<commit_message>
new products & plugins
</commit_message>
<xml_diff>
--- a/wp-content/uploads/wpallimport/files/6xxx-pillows.xlsx
+++ b/wp-content/uploads/wpallimport/files/6xxx-pillows.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\www\_open_server\OSPanel\domains\manuale_mebel\_tmp\import_catalog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\openserver\OpenServer\domains\manuale-mebel\wp-content\uploads\wpallimport\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D3F2BCD-1517-4C70-B0C1-9AE7CA18EEB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3000" windowWidth="28800" windowHeight="12420" activeTab="1"/>
+    <workbookView xWindow="20370" yWindow="-4350" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="сhairs" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="pillows" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="41">
   <si>
     <t>id</t>
   </si>
@@ -112,27 +112,6 @@
   </si>
   <si>
     <t>Подушки</t>
-  </si>
-  <si>
-    <t>1.jpeg</t>
-  </si>
-  <si>
-    <t>5.jpeg</t>
-  </si>
-  <si>
-    <t>4.jpeg</t>
-  </si>
-  <si>
-    <t>3.jpeg</t>
-  </si>
-  <si>
-    <t>2.jpeg</t>
-  </si>
-  <si>
-    <t>/</t>
-  </si>
-  <si>
-    <t>,</t>
   </si>
   <si>
     <t>6001/1.jpeg,6001/2.jpeg,6001/3.jpeg,6001/4.jpeg,6001/5.jpeg</t>
@@ -174,7 +153,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -252,7 +231,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -284,7 +263,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1032" name="AutoShape 8" descr="data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAH4AAACpCAYAAADtGIkfAAAgAElEQVR4Xoy9B5xkZZU+/NxbuarzdE9ghmECQ85REBQURER0EcOiIobVNbCGxV1Zlb9gWHPcNaC7ZteAeV0TuigrigTJGSaHzqm64q177/d7nvO+1TXjhq+VX/d0V9269z3vSc95znmDeM8v0iBXBPIFdLIV5MpHQl9paN//l6+p6Qn84qYb8fh0C/ONCHESIE6AqN1BHMdot9tI2hHSJMHfvuBsTE9PYcOGQxBkAoRpVt8DAGEYIpfLIo4TRFEbaQoEQaD/0jTVf/yZX9lsBplMFu12S6/zd2l/D9BqNTE0NKT3RFEH/HUripDJZPQzX5MkMVqtNjKZUNfgNYMgRBxFyOfzem8ul0MnjpDV++xT2lEbhXxePydJ0l2ZJOH92bWrCwsYHBxEgtieIYXWIghD7NyxA+vWrdP7/LNpqZEgRYQw5WcFuq+7H92JL/7oN4iRQavdRJQESHkdvp43zXtAqPsIwoz9Lg20hvy8OE3sd0kHnVYdmRR4/TlrsGHzIShmQwSd3T9Lg3wJcaEfmf71CDH8/1vwSGPc9F+/wV1b92GiGqERUeApkjhFq9XSwqdRB5kwwNUveZoWh/cSRTEenmjhqIMKKOQLXaF4IXMhuRm8wCmYTifWElEI2awJXgtoa6DXc9GiKNLfC4WCNh5/1+509Bn+q9PpIAxto/jP4PspeL6Oi1kqlbRBHn74IQwODWHVylW6Lu+hdyPaz3avS0tVlApF/RxmA91Txv2N10y4iXs2DBckoYJELQk+ifgwKTpJipmFRWzdtRdxkMFCE/jDn+7DUjOVUP3GS4MM78Z9PpAm/HsCrh+3kjYcYsSthhTwjecdjPUb16GUzyFo7fx5GlQGkR1ZiQSjyCQVJNSKNEQm5NI0uL1thdMiEPI7F8BWvV6r4ds//TkeH6+hHrURdfiB1LZI/4UIkEljvPXF5yFjSotWs45H907hsINWI05iLTQXmQu2YsUKUDBczGazgUKhqAWnJdDu5mJJw/zC2kW9heDDNptNXWdpaUmay/fZxuB/QCehZYm618tns3p/o9FAuVzWzybkRNeQ5gQBqtUq5mZntaEP3XIo+vv69DfejwkgQODuLUk67r6cNtIGJAnSBJifn9dreW96T5ggE4bI5mzT8TPnFmt4+PHtKA8MYs/EHAJa5CTA7Xc/iKUm7UkHtJeUU5gmiCmrGIhiW0d+ju4rTZC0KcMUf/XkMRx+xCbk+drFvb9Pk2I/qs0YhTiDXHMJmaSJfK6KrKxHKjMVZFPE5RFkBs+QMJfVLcUvf30jbn1sHLO1lsx9p5NIeFqUToww6eDvXnweb1M3045byCY5IJcijrzJ5AImKBaLWlgKkAvDf/dqqjf5XtDalE7j+Z2fy+sMDAxIUDTdFDq3MDfP0lJNz5TPF2SVKGhqJc0rtYXfqfVmIRJtBm+WeV95aovbQP5e+Ll8favdRl5uqI1s1txDQK2UVTBLwbXhpvPmWvcWxLrHMEy10WdmZvD49p1otGNkiyXsGp9F3GohXwTma21Umxk8+NhWtOIYowPDWDM6gHse2wagiKhjG5pOkMrEfyNqydS//IxRHH3sYcjRDV3zgY+klUoFU1NTyKQBchmglC9goD+LF55/LIbzixJ8JsigU8gju/J8hCltdtC1s61OHf/ybzdgz3yMatsEyC9qHn/OJAmuvuxp2Ll3L7Zt3YrNmzfioDVrzBXQLIY0uSZe+vp220wuzTW/+Jo4AIpJqof1LoEbI5PLaYNMTU3KHVTKJUTtSIKnkVpcXESYzWgD+c1CM9hstmTJKHh/v7wHCl4mmsIPAyzMzyPP+wiARqOJUqko7XdbH7EzqYVsQZvOW7Ukjc2sh1kkaYIwzwfMShHA2CPNIU4jPV8my+vxirYpOnGMhx57FAky+nwa93VrViMMUuwen8DCUoRCuSLXOr57CusPGcbCUoIbb3scsbM0iUx+jDjifXTQhyVcevpBOP7YI5Cjdfra93+cTk5OIZvPYXF2Dq1WHZ1mC83aEi668Ew8ZRMvkKATtVBZuw6obAJwsAu2nLTSGD//9S9x1+PjmKjTZ1mA4bUvm6b4+xedi3sffACDAwOYm52RgLm7qZGjoysUsMnP0i8FAbgZzbS7YCbsIBMtIc1YDOKDuXyxoJ/r9Tqq1UWUSyXEHXMfaWwWhM9GQVNb+RkdBXctFPMFZw32DyYtwMogl8mgVltCJpuRsKn9vGfeEy0X/TEFz/9nwxw6nagr+JSCp6Zn6EZChNkYxSjB1h/+AgPnn4MiN5CWzwJDfiaFVqvVkM/lUGs3MTs7q/UqlQoI6Q6RYseOPRgaGcHs4iJ27NiNeq2N4VWjCKI2vvrLe+UAJHSa+JhrEKPTbmEk38alpx2E4449HJk0QfCOD34kzYQZNFtNLRhVr6+QRy7I4PynHI/jBsaRBDk020sY3rQZcaUf2cxJ7qadEQ5Mw7/89e/gvskFNNsddCLz9RRAFhHeetkzcMedt6Ovrw+7duzEMcccI+HXanUJmQLx36npWgi3CWgRGlOPopx+G8mKd7hg0KL+TC4rTeQmu+22P+KUk09BTjEBfawFiabRAcplBmyJgj0KfqBc0bVCxg30i4r/GEMkev4AKVrtlhbcgsUIWZnkEI12w3Q0yaGDBKWcuRMf/EnwykKyCOlKqNWdNh79yBew+nUv12sz2by0ks/HTfOlL/4Lzj77LKxcOYpyJY9cJq+sIuq0XWzEOCdFua+CyalJHLJ2LRYbEXbu2YeJyVk8vGMav3lwL8K4DoQ5cylUgqiDVaU2XnTWRmzZvB6gqX/Lu96tfddxfpVBRtxsYMuG9TjkkEOwAtM47pAYzVaKVUccDpQqCDIbkIYruhE1nODrrSo+8cUfYu98FREFrwAjQSGu400vfibuvudupTrc0f19/RI0NZWawZ0+NjaKYrHkAjgL5LiQXPBcPo9Mu4qwOOjMv5QQoYvwd+zYidnZGQwPDWPzpk363Hq9oVSNLoAmPJfLY/v2bZhfXER/fz+2bNxk6ZpiAKDdifDJb/wSrX33YsXgEAYH+7VBR8dGkQYBRkZG5AYp+HZswhifGUchl8FAedRlCpa5cHEVIHJzcrMkKZoZoDYxhU6mgAwySNKONhQ3CTfiXXfejqOOOlKbJJ/PoL/Sp+C31WxZzBGYBeOO4vfFhSrmag1MTM4pGJycmMSP/vgomkwL40Qug66FmdWmkSxedPZGrD94NeK4jeA1V70t7fo4mp2UMVeMSy65CFOT0+jEAR579HE866zNOOWofgSFQYSVAoLcJgTpMJIgRqCcn0Jq45Zbb8cPb74X1VaLKaQWYTDTxute+EzUmnVF6ktVi7Z37NiBww8/HIWCBWC9QqcGc+GoEbx2LhMqIOPvvannxmCEzvu/7757sbhYVZ59+mmn6TWNVltWI+lESs8ovPvvu0+awLs9+sgjZL658crlCh7cuQ8f/Pb9uPJpwxgaGMTu3bt0X6vXrMGGTRtldnPZnEy/rpsk+PUTX8KmwnOwbk0/skFemRAjfL6v2WigzRRRAVyAb/3bN7B+06FoNprIFYq63pFHHYn60pI28ezsJFaMjiBIEzA2NHdYQLvTRtzpoES3FobIZ/Nah4WFRSzUm3j0iZ2oVhuoN5r4/UO7MbOUIHJ5fNrpIG5GOPfoEZx34joMDw8giSMEL3/jW1Lmf0p5GNgAGKoU8IJLn4PFhTrjEH3Iw48+imIY4ZXPPQKVTBXIZpDk1yE3cjLSJI8gJKDCuH0JH/rcd7BzugFaKKYTo6UAr7rk6Wi2qIFZmTVqH687NzdrQVmlguFh+m8LvJjSTExMaAE3bNigTKJSKTvfYj6RWkCgghbhN7/5DdasWYMjDj9cWsznec+n78RVf30csi7Fmp6dxbZt2+S7+d7jjz3GNkFAN1DGzp3bsXdqHpkkUrBLa8QgkYIfWbFC1oqWwjIASxt/PfV5bK6eg77RMdTm5pANs9rU3EzNVgsbN2xQlL5z507s2bsX+UJZcU2xVEa+kMehhx6K+lJVlmmxOodyOY8iQSKmtKHhE8wQCsUC6JK56bKZrCxBbamBbbv2YGJmEVGUYGZuHg/smsPjuxgQZtGJmR01iTzh5ecfipMPX60MJqHGv/T1f5MqCGDixwgzAM44+TgcfdTh+NOf7kMUmy9dvWY1JidnMTG1B1f+xVEYqt2PTjNC/3FPQWbkFAQMurjL0EBUn8XVn/oZlhqUfILNa4bx/HNP1s3uZ6eVH0vWWkjmt6NjY2g06hgfn8CePXtw+umnC/EbHRntWgYfnevtYYg/3vZH7Nu3D+vXr8eJJ5wgMyNrkBIPyCKJIgnxlj/8QUIblhkfxNFHHWnoYpxICLV6DVMzM6gtLEqo2VxOm4jBICP7NavXoFwpy6r4lOy+Jx7AVP4OtKt1HDN4EVavXG2pXauFdquFSl+ffvaYAnEOC+kYzWcl8Fp1Ud/n52cQZlJUaJ06bX3G4OAACnlmL4w5LPenJSDwMzk9h30T01hqJVhcrGF8cgq3P7wLaVBEGrcw2D+ING6inM/gvFPWY/3YANI4EpoXvPi1b0gVfSaxfEIuCHDB08/C6NAQaswj832YmJzA1MQEVq1cqZ3M6PySsw7HxuqvcfBp5wLZPLKrTgXKa5nEIY2X8MjjM/j4N25Gp5PijKNW45xTjrHgURmmhyzNT/svRvaz83PSKm4ELiDTNAaAK0dHLUVzUK5/D9Gr399yCwYG++X3DtuyRWkU79NchWUY//7vP0EUd1Cv1zDYP4CnPOUpyiYoeCKJDPwWFxcU+XNDcSP4qJt4ALV21SoKNZR18HDw4vwCwlIOeRCCphu2TdeOLYAsl/oUv/B9yjSE5Pn9bz8060tKjaNmA5kcIe+m5FEp5DA6MqwUVprPjZjNal0InO0dn8DiUh3bd41jZmZOIE0rTvDYIw+jkxIW5/qmmJlbxBuveC5WDPUjAP1vB8FLXnsl41kkxMi5C9MYFzz9yRjs68PIyoPw3e//BzZs2IhDN29CjYjS3Bymp/ZhamoGpx67BRcdsYS+0RGkURbZkTUIhtfL58edFn5ww0+wYwY49YQTsfagtUhSQqghgh7s3YMjFBQfqMHswqVhtADUFP5+zSoPmdqiefDE49U/+tEP8OxnPxv5XFYC88ieoYIJvvWtb6HWaMjMjgwN41nPehYKhZwEz6zANhtNo48tLLjsBYxmZmdRKpYk+IWFeW20pVYN/YVBBGmbS4rQSbUZtXXtSrlProvXYXyTybEWYICPNF/+nJrM7AIIMwSRAqFrvH4hl0Olr4yQbq3TkQvqRJHwiUa7hXY7xsTMLDpxCjrq3Xt2Y+v2HXh8zzxajRAnHbcF//mHu3DVZWdhzdgIQOyAgn/xq/86ZSrD3cE8cmSwgjNOPVFARTabx969M7jngYfR11/BYYceqhvs6yvj8ccex/S+Pdi0biVe+pQKiuWKHqCZFtC3+kiAaU4c4QvfugWnn36StJU5pfd/HrmSBXA4O39eqFZdsGXQKYMvoW8Cd3LL5qHnJ+HXjJwd2KN0zL2Wf7vpppvw2GOPKTikmTzuuOOwZcsW9Pf3KY1lbYGL3GzWXexBvD/X3aCG1IUuj7eoPopalm5mrEbA/6TRLjefXZiXxq8YGtFmaneIT1hsYM/sN1WAbIbWKVQAawheiDyBtEIO5WIBhUoRGVqiqI09u3ejVmtYLYM+P8xgYWlJiCQ3RL3Zxt7xSXzz5/diurpEDBdRJ8FVzz0MGzYejBzRUwr+Ra96dUp/YVqS4JgjDsWmQw6SqcvnCgizBfz+1rtRb9RQUjCyCZVyUbs+G7SRaczj2KE9GB4cRJhnKpZFFORRXrEJIQpYbLewb5GbyBbS4NP9v3o1a3xy0upVSYKxsTEtpNA9p+W9xRvTGHst/feTzzijK4ReTb355pu18ShcCpzvocaMrliJhx95GIcddqhuiJAufa3/UnlC92z+la7QinCEf1vaXNS6YqHgAB3TYH72vfc/jF07d+Jp55wrX01s3XCJ5Y3iP4eCp0JRcQw5zCAfpig6wRcrRYT5HJJ2C1sffxyZXEHK4HEAru327dsFz/J384s1XPtPN6Da7iCKAuTTCK89fz0OPWIL8gqeawhe/TdvTGlOozhCmMQ46fijEMcRWq7QsXbtwSoQ0Fc1G3Xcc89d2gAEYsaGB3F05hEUC8BA/wDy5SKCXB5BNod6M8Dw6AYEuT5MN/Nox3l0gixCpEKOzF57HIi733zgdR/5uNIyBmMffc81KBWLLnWCgJCudXDYAS/zuc9dj5e//Ar5P7+JPOwqH9qkSWzJT1NYvHeLzjN44RWvxre+8gUhY9RMvzFlkVTBo3ZyMwQy3VbetZ/9a7278huR36uNJv54+20487TT9Fr/5QtNvJ6hkgmymUSCzGWySv0YzdNjlfM5rXWhUkCmkEentqQUOFfIo9mIUHHPkMmwfgCMj09qA9JFvulD30A7YqU0QSbo4BXnrMfhmw9W4Kilv/B5z025GOvWrlVAcfDa1ejvryh9mp2bRZxE6BCISc2sEKTsL1eUfo0M9ePQ1h0Y6K8oTy6UiwhzRJtyCIoVtNopBobXIghLePvHb8DehTb+8tLn4vgjN5omOcxbwhKgkeA1b/8AOiHTwgD/dPWVCAPnHhJfj/eVQds8fMhf//o/8bznXaJrMrWzwoyle94ieKEIPnUC5ee+7K+vxJev/2cBLMTK9xOig1It9bCSrxe2TwO9Zel1XYK4EeC+B+7HkVu2KENYtnQs1tiuN+g3RiFv0XpWpjsE91kuG0jwMvXlAggQRPUlaXa1XsPw0KiCPX6x8ENwaXpmBq1mW3HYWz78TTRbHcRRG/l8gsvPXodNB6/D8KALkJ/z/EvTgcE+HLppA4rFAlaODQk0YJCkuncUK9qtLi65Wm+iXDKfy2NkcAibc7sxEFRRYP7JSleGwVUWGZZTcwV00gwKfSMIikO4/LrvoFGrIwlYnkww2NePjetW44Lzn4Yth6zDJ6//Mh7dPQ7kCtoI1175SgyVgLjREkKnyJZAKgkU4H1VMbhiGPNzCxjq7/szF+Kj+t4/eEFp6VPgjf/w//Cpj7wfiCPVnVi4sYoagSl7J7+FQQatqOW0ny9nqhjYexwxQ9kRU9ogRKsd4Ikd2+Q2ezV++V6MEEIrUypmtFnzJEi4cnM+E5hlLRaQKxPCjtGq1bFt+3ZkCzlQy5tNuqYsgjCLUqmCMJNDNpfFtq3b8I4PfQHVdgYED1fkU1xw8lqs33AQBomM8tkvu+Kl6dp1q7FuzRoMDvQpcFMli/wOmjWmBQxsmg3ML8wrNWm1Y5nKfBhg3Wg/VlbvRLaYRblS0aLxBmju+RC5Yh+QZJAvD2O82Ye//8x/oBU1EGYI+ph5lwYSnQpyAjYCFm8yKY5auwrFTIJmdQnPe9bTtdkCvjYT4t0f+xz27NmNv7jwAlx0wTnIWu7lavWe1cPCiVUAewUuoVNoCPG17/8HfnrLHei0G8jEEforZRxzxGY8/aln47CN683KxTHe+9FP4pqr3uSw9VAFIC6gIfIGTfOzmOb9/k/34f7Hd+D8M5+EjesZpyxXLL3lYebCzUXLUSnnpGw5MpPCjKGY2UD5e4WxVoUwbQeNpSoeeuRhlPv6FHizFkJLiyCHThRjaHgEYdYRWDJZdBAik3Z0j1a0S5D4MvGr/+av0vUHr8f61atlvivlfJd+ZP7NLsSImNt7sbqoaJVwJMuEQ5UK1jbuRCYXWuUqzzwzQMjiX5hBm/VUokhBHmvWH4of/G4r/uO27dpYbW4qMEJuW82fhZT+QcGwjNL5+7hZQ9xuId9ewrVvfS1ymQI+/vkv4eFd4+4+aWEiHLpuFd706ivQV3CEiwTohFZmpZCotywtKyf2QSECXPPxz2PP1Jxpdmo0MRIzGGN0WE7lrbCQggBf/uS7tUlrrOk7nMCTKch5EXMoCfHCt7xL5eIrX/YSrBstY3Z6BgN9BdUuKIRGo4Xdu8exa/dOvPB5F2KgXEahyHWzjIHxbzEXopjPolzIIlcqIUg6aDWXcN999yNXLiIT5pB1sVcmVxGoVF2qyn1QcbmpGezJUjIY9eCZMznB31z1uvToo47C6NCIBJ/PmW/0VS2PmXMn+jIq38uSIdOf1cEsGrvuwPCKYb2n1N8H1qLDIMekFDFyKBT7URwYQTbH2AG47ut/xI5FFnEIJpgtJZbA6DTPYM5CeTFWmAlk00Rwbzlp4bCDBvGH+7eDdLFcPsccVItJGJiVqDBu4Z1vfT0OWTmCX9z8R9x88+3YO79g1y8W0CYvkFS0NEGGcUsh362tJ6nxANBuyVfyXgnEEOPnfeTiOlqdWEAUOQkK1LKM6Gm1DIXMs9LJIkyWVTWWsyNRusJOAykrZtT0hG4kRSZMcP27r8Lw0ADyBa45sX76+ACFLE19TqhbtmAaPzW5TzB2QjdQLIPgVS5bRCZrha35+TndA91th7uMMQq5BdmsXJLnMcgCXv3Ov01POP4E9A/0qUzpmSI+L2XgoAjZ8ceIGQ8OjSDMpajNTCC751YsTe+WyeEN5ooFpAysuG2zBWRyZWRyJYT5MoqlfoRhFnGYw1VfuAW1CLpBCo4mnOaOJsyDebwHkidZQ0ijlrFhWGpkvuwCIZp9sktYcTKwhiRP4u+GS/B31A5FzTkSOwzdEsMna+VfQruMri11C7nGiNp1wdc0xdyE/EyRJDr2OX4RubAiXDhCYTZfVArMjED3w43SInBl+TtfqwJP3AFD5X++5rUYGBg03oDz8Uzr8rkMSrksysUssvmsyBSsMywsVeWCc7miaFf86L6hYQWM5CNQu8WFSN3n0fX2pNDdNPcfP/Cu9Oijj0bfQAVFLnpgCJonUdCP6I3coSI65rBipB/ZzhxytX2IOouo7duL6clxjK0cQ4YFCNa9aSZzXARWxXISfC5fRqFAn5TBTKeED33vbrFd6Q2I8qt2DeKelrrJF4fmn5NO0y28ESy4g1ms4AMGcYo0dsGW6E0mSNYJjD3kijq5vOruZAGrPiC+Gz8nNMzesWnQiUU8YZbD12nzOOSMfpkBmQiNciEeRXS8O2U+WQQutYxliex++NncuAS2WDEMgwSf+ofXYHhkRByCbM7cFO+3kM9K8KWC/Z4b7oEHHkA7jkX+LJcHuDgqjBl7LUB1adEwEJZkewTfi5P4+w2++rXr01WrV4vlwaqV1ziCFdqhpOrStBGhCjMkD2HjaFu8vGa9jrjdRNysYs9jD2JguB8ZmuACNZ10JQYreaRBCWE2L7+XLw0gn+tDjDZ+c/du/OC+mvBjZlOMSOlDpXUUvMyhOSWaRgrn0IP6sXXfEpKQ6R+lZygYo3wKRCogjXRsU2k8HTWZKYzWtR+M/0ZPyOditcuBWKxokc2ijeBJoEnarfi1Wg0XD9iG7AaOzl0pLuKzhgy+YrRbNbMQ3Ci0KjT9LuAM0wiffsdfYWCgT4hhzmt8wOAui3whlLknqBS12rjznrtQHuzH4OCQTDyYriZAo93R91p9SXEXuX9MSRhBJQ5V7Kad+n2A4Mc/+U5KQCOXz4hkwN3vH0j+nTCj427HaQfFxm5k2nPYsPEQRMSK63VE7Rr2Pf4QKgMVJEEWBW5ZMkizOSAoSvgQm4QBSQkD/YMIM+TlRPjkz7Zh20wTqk7QVwZMVag1zu+H1CQgK9Od4NzjNuC3D+xyTGBHLdZdG3tIbF2nkWTL2LMAMS1DYAJmakaBRdwkjCXSZZKmuAmuTE36uEyzYyZRGXRtugrHCtbN9RSaqIXc+Lwjlpup8ZaimZknN5/aLvgaMT76lpeif8BKtdzkSlkp+FwW+XwokkcumxEWQB4e01fB3glzfqDFmCXOY3qpij2zc5iYmRNPj7WCyZlFTE3PaN2EzjLnT0l3zyC48Vc/Tum3izkLSLxv5wsZFPDqeQoOQH3mUQwkS4iSNhb2PobDjzsJcZpFVF/Avom9QGkE+8IxzHcsKm52OjK7LIIwJ+bNczGYEkqzyRlfrKoQwyCKpVLyyK3yFWL16tWCbVetWiWK0Y7tE2i3UmTDMgiRkGxA16SFdSVaU2fXTOCid5pDWS9uD2/JaBIpdPpD+VwK1Qo6PjXzDFlqqzYV1yS0ErIIoO493WvyNY73T+toG8SII8IFGE+0m+b34wh92Rj/+IbLMDRQUVWQ68/r5sIApTwFTnOfU7DXaNZw74MPYcXQCmT7BjDZifGr/7odv/j5r7CwuKh7bjZaiq083Zv3q/RQjSP2DFIoupxb/vDrlB9AOpQ3W3yDSrREk/IFFLIhGgsz6M83sDQzjrSzhKWp3WB4Mrn6RDyydwaTM7NYmJ4WLNpqkDHCsqpl1wGjJUdOZIzAxgOqCYMaMlomJicRODIGF4qfS0TO4EvL9WnGy+VB9I0MYGx0NTYefgRWrdmARx7eiUZEDJ3mXi0SXcFzc7HkaigZwRZWDU1oKrSoGhd3N4AyBLo2x67hhvELpss6gEaBo29scBU2a6rgpjMLqTuReTerwcIIf8fYQTy4pIOV/UW84xUXm+ALRgRlbJPNBMrj89kcClTGDNCoV/HYvgmMHH0qrv+3b+Kmn/wUzaUakpibqS16FtNgGnLdpweedE1bG/8l2Pu2229OuSuIEgmWJFWnY61D9LnFfBHtZhXlPJDEVTSJ4i1MYms8jDu27sbM9CTI0m3WG8rzSXpQaZJa6FKIgCkSF5sgBzlkDeuCUTqmbhLyAai9xgX3xAziBTSBSptUuOH9RdIkslsYMwyvXIGD1q3H0aeciU6SwfT0IoKYKZsBJGCwaF5N2YMv+lBI0liCMNRALprzvd02JII0PW1cerFr6uBr+JV4eM9bFwnb/KhF/wbskC9HgXdY/ubnJh0cubYff/OXF6GvUjIGsKvO0UUJwMmhtTQAACAASURBVMnS7zM/A+qDa/GjO+/Ad7/4RSxOT6M6tyRhE71jzKB7UZxhULDhLz2Bp3sOX/0L/njbzSkrcTmmR2J0UvAdVYoYZbcaTRy0ZhSt9hLSxhyqrQQ/fGQntj7+BHbu2KViDh8iH2bRYTWo1VavF4kN9CX+i5pLIERmNKILMHap98Eyxu5GuVA+q+DfvQYyWOli4u5B+HTtVhv5QgnDB43h8GOPw4bNR2PX3mmkCWlGXATD9wn3d3NZ19JkqRU1uCPfq9cR/OFiOizBP4OYSq5nwN+HzwR8XYBK7zeUrbxzEdlQkCvXlqkc1+ysI1fiZRefp3o7LS7jWaGdxEyyxO/p5/OYHjgIn//eDbjlxz9WQN1qNlBfaqJea1hmwazF1ROM9r1MF19Wc2cRfX3k97felAouDPkhbDeyBgfGZwsLCzh43TraAbSjOqr1Or53z0N47MGHsG96EvW5qpkR+lpqRxoKsFhYnFckOjRozYsKimxFtC1ljrgBGEGLlNhCqVDosm60GZyvtZ1sixfzvU6jFMn3PCT3GO89E2aRKRVxzMkn4fjTnopHH92joE60aaVUbocpTTOzTpaQNmTbCBPmmy1OULDnzCbvn7IkV4GsIAV+jlhpG8HKjbpfFzjK1MsCpOqGMaoXsYEEr3j2GTjz6E2oVAhG5RWRM0dnUpvPBsrfp4fX4Gs//BF+8Z1v63lb1RqYWSxVG0g6ZlloKUzY5t+9lRKwxKyFn66mFXNxMvW33/m7VACNfEtGwdxAqYJGbQnDI/2Wr6YdAS3fvO123HHbXZidmUCtWrWOGknGkSmcxs7PzWgB+ojiuQVQlbOnGdIvKv9OCJMwr1AnSlDWzW7UUDHv5ykkBkl6TMtZXb+sqMxOQ/3DFQf7cNqZT8bw6i0Yn6wJE0ji5cWhn+X1fDCXOFPPq1PjPa/fkD7g4tMOw3Aphxt++wCa7Eejm0jNaoWsx9HfuoYNWgLhDS4IzKYBWu2aijtJRFcX4W1XXIzD1q1EX39ZcY1RpcgoNnpVe916fOM3v8F3P/tZ1BaqhgoyaK7VQeNET8brdxtCVX1ZFrA2rCd8sMdOWY6hecG2HQ+nytPNXuDxJ57A0YcfoXowIUxT1A4e2LMLN/z2Fuza+oTo0Z1WJLSNC5QLrSDDYExtU0xX2EjhCjVSBEGvy3mPj4yJhjEIpPb5WrUE3omF5JnGEZQx7bTXE41yLdRsfHAVLW/GTUUNDczm81ixcgVOOvNszNbLruHTbyrfsGnBIz/TbzSfx1twB1TyKT74mmcp335g6y58/IbfWZSeWPA0UExx9tGbMTg0ALJvdkzXcPeje9FJXJFILeANtJsNVQJzYYLrXvd8rBoZRH9f2bh0LgilArI28rXHHsO3P3s9gnobs9UF631okyzJFJNt07auXmFo0cTjd7QuAW8eCEnNTbJ2IcewbeuDMn584F27t+PILWSjLGtbSsJDp4Mv/e5W3PmnP2FpsYrFuVlpL1E9+TYX6PhArN1q6Ca5YqwZq0ecrcmwuEFsWxclCxGLY3HLuNhWwrTAiF/LdW+XirkHUBqnaot1wfhWKh9t+9hAGiQwpIC1h23E5iPOxkw1Ul4fKge21IqWjXi/zGVkm4zBqQI0JHjds0/BiUdsEMBF3ttbPvNTcQUOO2gIVz7/PAz0FY1k4hDHWr2O93zlF3hk15Q2ra4dR4rASW8uFXO47lUXqWuGtHFDLRkQk4oVYm5sNf7hfe/B1ONPoF5toLG4hEg0MWtKZdm6G++4YpoXfJeswt/njJwiM2+9WsaDePSRe9K5+XmsX7MGCCx/FnTioMqApcMgwAd+8GPsfvwJzM3MoN2oi03q4dzeHnANFiCCRi3nYjKQ4W5nBymBA0er9bvS/5uoIXljZMowyzDs3ARP7fZt5f6BfdVQ+DbNGbn0Dnvw1/RWhdaHPpQo0Nia1TjhjAswOWtAjG16mnWn9Ywj4tRtVFcoCgNc9+Iz0NdP1GxYz/APn/gOLnv2Kdi4akiVSNKoSZfig6saFkW48iNfxu6ZljYPg150Wog7LP7EKJWL+H8vvxCrVq2Uj1ddnSRMRuO5DH40OYWvffjDyKUhlhZrmJ+ZU3Acta0TNqZ/d5aOz6D18B7Qde/qn+x/cJCzBG/BAIId2+53Pt7Ff0w7HFNUQUkSoBp38I7PfwFRvan8ul23smTiWpx1QZcoehCIQmfpVakSc2kGLs6HEV4VE0abzOWdaqNqSPs8iMRqYLPe7sKdPupXHaDXnCk1dJvK5azd6N3FCXzkTDY0GHRwAOdc9Jd4YjvhYm4qq6AJ+KHQ9R/dHwXPew9w7UvPRH9lQIUUami7k8itsXTKz+qrlJV6Gb0a4iy88rp/xXStZe1EHSvwsGWZ3/vKeVz3hhdibGRIVVG5L7c+gysPwT/dehN+8JnP6P6qMwtoLbHjJ2PDHshWcmml4hkH0BizyBWaHALLTKZbZHOMJHEHd+14kFVHV6PmbjI/4YVPwd83PYWPff5fZY7n5+ZkchTYREZGoKaxYCKBqJKX0YL5luGUwxKSjh7MdhzfZ2M7WEnTZ6n6xc+3yNkHcHFkkasEaVmquXBXePGbRDEhNcBPvnCsV6/9phXcIHI4GFq1CqefdwG2b20gn83gnGMPkRn/7n/dxZKhLayvwgXAu192FsrFigRPIVHgCgLZxMh6OmOOuC0XwveOT8/gTf/8E3EXhAa2WNjpICVyl3YwUAxx7etfqALNgOfOuecc2nQMPvbv38RP/vXLlAZm9hHgksd1LsjRz3rmAsiUZ4ysaWtlcDV9vA98icR2K5+7dz6QygcIraLf7MV4yBMP8YddO3D9176h/LK2uIimIw9GrUj1cC6l0DUKm4tSKNrCEaZkBCn/Sf5XR68hN73XHHOz1KqkdrnUR8iYE7KCq9AKHMs7Qu/3voubVQ/sQRS3v2je/UQMml5x113vO987vGoYz3nui5GPs3jSYSsxumIIP7nlQfz89ifkl3NphNEVfQg6EV777FPEFciRaCJuQkEAlPAOdSDF6sSp1uoWOacpds/U8Jnv/Qbjc0TW2GjSRqfFGT8RBgvAu15Hwa/A0EC/TcfgtqcVXHsoXnf1mzG5fatKzlN7JtHh3IGOwcm+zNoVLhXJTwhxZFDx7DXQwp7ZK7JiCf6egtcOcRUkXwZ1ayfB/+qhB/HV730fGbJLG03l96VyWRE/YUMPanAgAS9M02XRsHWMdtqRmjFs8gQrgMbn4xdNF+MC+kDW232TJFXarsF766mC9RAlfflYZt5tPrZNd+MIEhBcOsWF55qqGOKsAu3Ohk3r8fn3XgeNYBChsw0aeQFMCjzbyDgcgDV1wxCdFWIwB7aBM8hNMTXJoQVVDV/Khnm0GzU8MVnFxFwTESNql3qxBFUuhDjs4DH10omHILIlkC2vwOLAClzygov07/pCFZ1mB20Ol2p7opdLZl1G42XmgzplG07wHAph7CbPHbQAO9i9/T4J3hcTlArqhYa6Maj/z4fux5e/+31ZBX6xyCL+eQx1frL/2uBJE1CxaItLTp5cAtOwTgdlNxjIm+dljSWJoGpUoR6Dw3TQz74hgdP8mQV9rO759mb/wIpJnCWggBmWW3rJoIj0Lr4vRSFfthjFggYce8KR+Ke3/r3VFBw6YN9tuJBCHocRMCAkoqaRCMp1m/pMVtHsy+BpFmvkXlzM0VvA6xZKHIrm75vSKY1swV21GVz5ssvlPmenpsCCe6tJi2kVSJE/3CaSiXdarfV0d2FO2PrzFN84S2DE0RDBrm33plbNMTOrFwtbtxunlm+dmsK7r79eo7zYfz49Pa0LksMWkbNOPyZcm5W1SIKXRlOQbvAAr1UgEcL5TW9R+JnUdGo+f2Z0T7fAtmUjL/ohRRYjdWnTLK0q1bL7VZroNibzYFW6OP6M07ESG8ZEU88qPI2z0kg+tWvHPvPME/G+173WWQubKME14OcRMeyicc6dMDKXSVfjlJl2GzbkNjvDFlcA8trWGzQ7jnVXG7VJMgWs2nQyfrvrYVzzt29WlD89OUX+F9qiSpu785u7m7Y5KrndiOvqcZiAXusKNZIZ14qbYPsTfzJT74TufYU3lwRdluIYV33sY9izaw9WjKyQORNAE2bEvo3qNk7MI2Z5ES4ziv797zTPxhcvyHdj2ZIkxowVaRrNpjB3sk206TizjTmcQ798dcsTNdQz59I3+XE/G8fh1EqpOJPGaYcWSUkE0zZHRhC1i6VMoNzfhysuex4uOpkNJS6ecOsiDXVAUrfjV1mLzQEy6Hg59LTgys3qcTvcv6Z7bTapOqSQm0XBbHkEJ552IX744O342LXv0maan5xGu2Fz+biBvUWWn3cWdVmbrTZgf7PmjO5XYAJn3CNTv/WxO/aL5gwNNRaMNgHBlzCDN33ww9ixcyf6Kn1inwqQcflqa8nmyfmgg2wer/FKP8IQfUxZAvpO02JW/riYziIKtrWCg2kaF0OQqcMCLE0xbdKmFI3bNpt2tcP0lwNEe61gaPc3EiK50RgzeOugZgfahlwGI6uGcd0rL8eqsgE3VoFzNWz304EIoyeKShP3Z2Toc+lQ7AeLDZQ1+c3gt0vQUUo2sPpobDzyqfjmrb/CZz/0QY1dmZ+YRrvZURWOFsBruy7hNJ2/M/KKZWTmEi2GkrZrjay+z79L45949Pb9BO/RnS7+y3AmCXHVJz+FHTt2mUA5k6bRQKlYUdNhxFzbTYOU5udC5IJQ06fYj81FZMrDpkBGwuz0ILmQr1XFS926ie1q23eiIkuPxKaxFE/+TNQsg2xlrknRJj6uoYVu0uMBdCNR8Xt64nxFjUGnf5+lPMARJxyGa156ETLUSEfA6DXRvaQLm79nFT1vgnutp35nXG5Xo3d7wAWtXY/sovK1R12MFasPwse/+Gn88IeMqYD5ySkkkbVs+U3vYyMGsvwitd1vCG/apRgug/EKwPsVY5iA138neAV33RZhUpECXPu5f8EjW7dK4H0D/TKRHkWrL9ZMu5wPCYwnpfStVMx3aT/lkk2x5AJzwyzn2AGWFmwciEG1ROIsImcngP8d8XTjsftq1HKRpGsJnDb5a+vhGR73jEZl4YJfrTpHlbQVRKnuEDeRLZbxgueci+c96ThZGwWBPdMovUXxwv4/v7Ms263ULTd2UOhe8N4qHHfmy9AulvDcv3yumjKrC1UsTs+ps9lrhH8uWVjH2OFoWD+mrbsONPU9FrHL//f4x4GC38+H6Kksgvz6D3+AX91+J/ZNTmPlihER9Kkt1NzZqTkJQ0T+lEOEbKJUg+PHOEdOXaaWRlhbVluRsebcudIqW6v4ZRUxC9i8pgkAcUQNPxOPVoAFE2M1G2BB089Ie7nO76ZfMo5wjFsjaFre6ytwvjpHAbA0zf759771FRjmbDqW5vTN3tNl3hxQl/ea7u/Zm3OBNu4f9gzuOiqp0nbbv/m8p5zzKuyLY1x8yYVI2x3DTJbaypq8Jve6VFpemfWsZVPe11NxVJ4mXOuCX+HzPRhG8PgjtxnE63DcA4M7H93f/8QT+MfPfRb7xqeENDHlZb5OwU5PzMgf2pgOju0IdeP0nTRRjNR9p6lpl6dsW+uxiBcy81bb94vnYwbTKm/q2aded6NOjTxiqZkPZJbnxskMujSG16LwhEp2HL5AUEn4dyR3w0IKcfNGp4VDDzsc1778Ik0IEYfAWQxtHIcNeJN7oHk3VpFx7Lw2+2zGx1tiHYnla7uCKdZJT389djTn8ILnPxedelvZUmOxDgJlPiXrjb+84PkZJlRvqYmeWvpLOSnO6Y5pdXHC/yR4v2M9hZQ6e8Xbr8bknnGR+VeMjarkyKDFplVbfkkiBunCNKNcNM1+4ZQot9i8GU8j5mf48aX8O6vaxBMOFLwewOHntPISpjRcW9YshWRqpeVljTfT6tunVWdz2YgXGrEDVhKXLUyKKG4jzGVw8bPOxAufdCJsAJ4Fe70MnD8TuIJIY+76Qpeyu57ah4tcZOks4+GfmXEkOOWcV2M8buOSSy9Wl+zE7n2qzJHZpC9qdU8rOF2WBW6ub8CGDysG8jELKdi9BTFqvnoi/2/Buy2QBnjde9+L6YlJ1BttteV2Qkb35JSRTsVBBqOYn19AqZRHu97UBAcxWVUAsRiAi0Vs3LTBEEMztQQnyJV3wEi3b8+CPbJNJHAVAARDIAxp1m3OjUYnyGotR/8+4PK+jhrPh+a24ZeqZq6+73237iVuS9Yjq0bxrle+EKP9JBwaC8i7pgNNe9ctuUaGLqPVW9NurOAYPb0ECsZHYQnHn3s5HlgYx2svv1xDlnZyXm2DzRd+MzlAxltnx67pFmnYs+i4CrbZrWdgOZay6p/WsVfwvQHRssZ7wQPXXP85PPjQw4hbxqAt9pUM3NCM+hhjK1eiVquqVZjATnNpSa1V9SUifSZ07ThXRyf6Z40PXviU3XIwxfuhpis3pbhcNUlpXcrJkHy9VarYR+bUwpENliNtmVJqhhtQLCF6mJobxY0oMbCIrNsYaSZALk1wxMlH4e2XPBMJ81ovfJ/f76fJPtbowQDE0LGClFHUjPcvSmRP+sshxtlwJU4454XYWp3Ei1/0fAl+z9YdaNVZOXRkDnLundnWWtBqGBnfSCeCqx3IJUw+g5C9DS7rkOvz6R0F37sjvL/v9a/ezPzyjtvxuS9/w7LTJEFf/6BAEuaM1Wodo2yhyqZi3HYaTTSX6IsLaDc5A4+948s0oS7o4Lhv9PMH+kx7Tw/BkprB4TBuSoVnk0p7e3y8sUwcO8VtBy2My2098GHgi6F/QtkI7XYJl4mme3AcyWUXnY3zTtwiq+ILJb1BXG+6p2v2cvV6wDF/T5aWmpn3eX2mshknPekCPLQ4gZc+7xIRR/bt2IW0nWoEqwJAFyAIqnYceW0gujONRjGkUabd+3xNyzAOo0y8h+T/O8FrZ/QM9vc3vGtiGld/7GNokM+dJOgfHNIN5Esl1JaaSvM42WpmchqDlT40qkuW57rOFAqeXz618IQLQp0+mjeTq080Abvac7cq5SY+9lokWROhaMZt90CP37wezu1uZpfOMeL2kbpZF2sX0+9oxrKhZr2vPmQjPvjaS01QnAbta/zO5HqLpXtydGsfzPXGAQdaUWsGseccXXcqNh5+Kn6382G84YorpNn7du1G2OHQZXYYWVTuhejxerOgoWb6UuNVYXCC1wAoR34xsGx5uNKf5fFeyH8meAVQKV7+9negsdRUF2uhVHInOXCEZoyBgSHBrgnZpBwQmMliaX5hGRNwJUW2QcvvyiVTUNY9Y4vEvWScd+1mZ+L9QtJskg7uLbsXJr/3gjzK9Z2Aeydg9UKdGhQgrGB5uD81nuwWfn6x5Kp7UQcnnnQs3vr8pyFhAEuouMubN+vXjd499O2kvHzfznKpIdQFgT7RC2Ks3fxUrDvkWPzbHf+J9//91UJMJ/ZMIMP5/4504S1ibwbmTbfGonhwxroQDFdx5p9TM2RlnaX5M8F7s3Wg4FVxSoFXvfNd6h1nixRBbqZz9DPs1SItScWWZlssXVbXmrVal51DhZF2OJ/LefDC792pE/74Ea6Zh0u94HtNqyyGI17sf2iApYP+iw0XfA4fsXdNsouC2XBh4IqnYBlvgMEqNy3rBmq7Zg09l8ObLr8Epx++1t7j8IflWMG1TrvY04J5l8FrQ7syc7cBw0f+/FuMw4+/GANjB+Mbt9yIT77rOmVDCzML6gTWejm+nA9Yl92FabH66RwobHgJXSLHprtBEY65a4qSLAd3+5khsTmWmyGW/5bic1//Fm659143FaMtrlkmzxw5oxnsNJXkp7MnnKldwBMZ2k2n4baQojVp5y0f9GP9ZHxI16Xrkbb/5lAkE6blrUyXvNb3+lrNv3flym6q5iZlmbl0ubnKrsuRtoKv0NURHKDE/J7CXrlyJT781iuQURVwmW/vJ2n6dTrQvNt9LWMBFoAsX4P0miNPuRylgWF89LtfxLev/4Lq8NXZqsUVztR3i1yyGm5su+M19Lo1tZ7J3xPSJtBlkT3nBHD+kCJ+H9X3Ct7vpt6gjxuVulptpXjLe9+thgIb/l9ANh9qxh13HevgnAUbtRqqH7Ma3G6Qg+5GjKo/3Z3M4HYhP88iV5q1XuybUzCXaWD+HjXT1VGfeMxIt1DjxqHZ/RsB06dy0pSeYr9lGGZ+fQrpFZQuzUWH1nDBOCWw4connHo8rnnxhSb2nqi+F9b97/L7XsFrI/QIngcRHfekVyLfN4D3f+Oz+P6XvoL6YhW1+bqUwbtf8fnUEk7XbVmO/8+ex9rSLO21vn/OxPGvMSjc4RqPPfzH/blWzkQtw3+2BqoMyc8neOW170Lc7KDW4I0lqPT1axIGT4KgeV+YnUfSbttkKJ2SEGkBPZZPky7SBf/ncHdNvhaH3wSvmXZuSrSgzq4sXErYZdosQ578DAIcytVpDTgqNJsTx603S/Edtt2mDBdc+nEhSiFdKZYLau3ONpuWNunNf/UiPO24TeikjAF8N+z+Gu03wn4Rv13VxTLELXyXTQfHnv1aZEtFvPOTH8BPv3ODMqOleTaX2nxc+3IVU5uNLlqV/u4yCV+UUXOGS/2ISfrfi1vAYhrP1fnfBN/VMHd+mvdb//CJT2DP1JR8PRejUCxr5CajevLp9uzcI+5Kq9HQOTcqtDgN87uXBRdj4jpSINMxtmARPOkhG0gj3YSpZY1f5ot30yEH3XrBy5wTruQGcaNWbJHoIhxh07mTLnjj0tRumCDNdBOtuufoNTE4Oop/uuYNqGTMTRyYvvln7NX85Y3gy7Q9pj6NcNLT/kYW6lNf+wL+5bOfQaNWQ7tu8/a94AlWeRTS8jKL6Ak7+9TWc+q8sBOljL5knopnL9i8V/B+d/aakO5iO43nv+fabbzlPe/TpEvWszmtqTzQJ23rHxjA3p27kXYiDdRv1xvIaEdyopnV5mlNBJa4yF34ucCpZbMuLXcVbvu558uf+uBOiuLDWqmV48eJ6pjfZ27PQoUGASjiNW2zcwNcW3NPV6tcjidhmC7p9dZfZ1VCC/5iHH/8Ubju5RcjzbigqtsHv0xqOdDk27+XBU/6uTZJ3MbJ578RnUwGV13zd7j5t7/B4gzZzHbGzeWXno+DRytYu3Ytthx+sjSf+AnHovArk7cDDLiOkZo3OqJ38/iS6mIVu3btxPjUtNZgdMWIxrsHjz5065+ZehmVnsHCvaaeP9Mkv+Kad0h41PhOJ0D/8KBQqpGRFRjfvU+CZ3GmVeOZZ4ZW+QYGCp5+U8CJS1XsnDTDnHvNI9l/vRG9F7/OaaPA09jGnrkqneBLsW6tVu+jenseG0fSi5z5wMtyca/BDvVzgRWbQvjF2IQ+ts5zdAb68YaXXIInH7vR4fcuqncuwt9nr8n/7wTvLdqJ571eJK7LX/ty7N69ExM7d+tcnA/+w1+jsTSuruX+8iBOOvlctOheOA3bATtqi3R1CmIZhgoukzbM+jlfryyXnTQHCt5H0YEt3oEab4fsxPi7D38M+2bm1KPNHJzjVGTys1nMzM6onMlyIjWe5XCBIq4Y4mqpsgJ21lsGhaLNZ9UZKgfUwL22q+/cgSbGqzNwg0ebLAekPZOhHWDRfWgXqBhGYOe8+SKP105P+jBugINhXVRurdNWziV5k6dPXn/t6zRShfN57b7deXvupn1N35t/g2z5xSPI3FSNNMAZF1yJJhJc8BcXolpbxPzEFJ739NNw7ilHKzvZu3cv2u0ETzvvL2y0W4YFsZY1RSqEtuYILU8P/iHShYO4FfASgeD3/03w+2m94FPpu4KSG/90L7763e+KK+fPNB0cGsYS83Z+eMeIGA1W55x5p6n3QZa5E+ukocayuyTmQAP23HVbq5fNpu+y8ILndcjtY0DpgzSZbwEX1o/HyFb5rzv7zaXConJzg7ISyE3D9/cya/wm8FG+ByIMjLHNEDV5wEEbp55wNN7xmud13ZQ/dsz34nvBd69Jp6TYhtVIA384NvbsZ70ZDXRw3nOfqfR3bnwSV73kAjVu0Idzrs2WLUfisCNONndDy8Jj3kQbk7S1bgKyZLKZvtHF+U3hu3pdJuAF3+vfe4M6X8mSeXQRqRinaYqXvfOdVp1rW55bKQ8Y9ZcTSjkgoVnXMIBC1qL9ZsOgXp9XMxU08gT71SC3wQKy9c7v3z3bTWV08C6DthBhjhg1I1gKuqPhTdQ4agg/Y+P6Q/T7J3bv0nc+QYFM4E4kgKRUKVvzB+/XUbcs6nbDC103Tm8qJmBJPspGnw8OD+Dav30lDls5pJGsjPIP9O0y94Ejk9AySPDGG6DP56HHZz3z9SCP6annPRWduIVocQEvOf9EFDJZNHiKRpzg0r94EZJMCXc99ATufPBe3PfEds0XaqlBdRlml3vTBDHWsK313GIcp/H8+ZEH/7AfEaPrTx2I0xW88416KLczrv70P2Pv7nHU1QiRiK9e4kmPBGg4cG9xHs1qTa1XFHK9VlVaVGBHiqNQ+SmWjI2I+ok73jMU2PPIfV+ZzFo2QKWYRV9fCUdsWounPOVMnHXqUZpLx5YvBWX8X8+YEl7zZzffieu//WNN6uJCsAlSvt2Z5WV83R5wWfPN9xuubwJM3TGqTBU3btmCj7z5cimdhhj3VO+6m8ALvksv94pEjU9x1oWvx2IS4YKLL8D87BQKnQinbFyFUilEK83h4aklVJsctJxBJ43sEAWlecQ+HATuXZvj01tKu4xzCDQLHHT7yAMH5PE96JaChG7o5wbEdcsnwHd++TP85Le/F1onDh1CTa6iH6HpnJ2e0lwZGh+mEJx/y9/zNTTBbe1U46bSzDdaNVWjSOvK02wHGR1Pyu5RNimefczBuOaNL0auWEa22G8bZL9wX2Fo128vM1qXq3V8psvecDWaHfo6etrlnOrLdQAAIABJREFUUyVoxs0aeaH7s++6oY6GBSt9SvxxqHRRCS574bPwgrNP0LHf+wvebWSX71NYxuJxfYc8H69TwbnPfAlum9qFv3rBJToAapAzfJMY2VUrdVgz14vsZimmKw9zvT1NWemby90Va4Dzh/O2Pjxjhz/buA7boA/ff+v+ZdmeAwB6BW94ke0C3TiAxyfGcd2nPt2tvtHskHdXLvcp6FuqLii4o49XvskTpjsWCFr0buNLKBa6DPo6FWs6ETauGcKpRx+FVZkW+ioZTcV68gXnoNTXr5mwYaGvSy1aFsufC94s2DK/3FLDBB/90vdxy+13q7ikESqOmOhNvQWLPqOwdNQqeNZBq0O1dW073rRvbAj/es2bNQv4QMHrda4L2QteZVKXiTQ6/XjqBZdhW20ef/mi56BVb2LLyjE8OrFP1TVyA3RapROumLLi6RlY1T1hROtMZI4HkCyPPekOqGQzhevuleC1XC5a9qdGdjnc3VV1gu+ZlUYm2LWf/5waLSi4Rt3OSunvH5QF0OTLZktNlS7YVGBF/63+OlKtoibWjo1gKBfgyU86Fcds2YSoVdcD7dqxC7XxvTa8MJvBEccfiU2bNyIln8zNxe2mTeLjOwxeW9ohjTpE0U2B8IvvovrPff9G/Ow3v9dG8C7OZgAZ1cprfm/MY0pj7dR+8BCZxwxKTzzpaFz7+svUb2iwrxVgzD0ai4auwCqCdm6u4vvsKpz5lOdgMm7iac94Cvt8sFSr2rkBpYIILzygkCCZGkRczq5Yh/UIxT3ugV3NPpfJWYDrqWou9uJhN9qu/5PgvU9d1qYe8KHH/33qhhtw59332KSodltBUqWfB+GWMD0xhYQDfHnkB4mYmVCb45gth+JVL70Mmw9ejdt+eyNKGaAl2lVq57W1Wf1b0oOPrBhFpZDF/Ow8CuUsTjnhKE3PDDlwWX2qjnPnTpdga7NFuAFml+rYPTGDJ3btwa6du/H4jr1a/MgJNYMQe+d4+JHx69XoofEtHk9YVohebIGLHDUtoGUBhCAWZVmq5PHuv/1rbDhoTFC1xQn+9Gsz+ewgVgbhLAp/Vxk7AkcfdxYerc7geZdchAyVqNUSNsIDhIsDA8gXy1izdr1AnJGVI1ixYrR7uBKHJmkABYmjUUcnWEQ80pTdSY4E09DcnQABEUhO5/CC7+5q59QP6JZ2Zn65YGBPFePGu+7B17//fXWnkBUqfD6bU8co/dLsvgkcdtBKXPv2v0eZGscFcQ2PRPTuuPVmhARIskTAlufMeoKCtKbTckeXt3Dc8UcjIjBT6dO8WBFn2XHSbOBHN96E2+5/RFOz5xc4vIEjWW0fdNpskDDNZuuxPUkWHNPKgMdAneWDE4Q0us1ghxQ57pqbasXOVf7dmK02pqUV1TE0PICvvu9q66qVK3DBoOPiJW76tbFmLfXadPRTMbZ6C+6c3o1XvPRFiBZr0vCxdWtw/AnH45o3vQOtbAGLSRNtXoeHKDLOIOdQQE5TgheLiC4kxz5CK+ho1Bt7DgXKaWqwgu//UfDLhYHl+vay1V8G++ZadXz4X76IfRMz6g8XQ4XDQfI20+bT11yDdSvYnWrvtvzdH/CT4t67b0UhZKQKneaktIqATj4vTIAFHg76L+RCVPpL2LD5YLTSAm689R48uGsvanEbDRI7NayYAmCDpAmEEueu9314nnZERJGLwaEMPJ2Kx4ISG9XwX1f77hZ12AnLmX3uqBYej8b3b39sG2rzi7bAAa/VUimUtfvXvfQv8Mwnn2LxkGsIUUbAymPkOABdMmmKE858Psr9Y3ikMY0rXnwZpsbHsXHzFnzn+i9isDyAxRCYojYrM2B3bIp21EQh5LFsAZpRE40kknvlBGveY7vdtJZwztbNZTVFVKd1c6Q6Q46H7vvDfsGdL10uI077C16+xEnRV6T/8StfxgMPPGoYfKOpAf2CU8MQ737Da3DcxoN79oyVZ81iJLj/3tt12jE5Y9wbGvTnqE9qiswVcffObdg6OYcmkS4e40VtijqIOHyJ6ZXNf3CsXetatSKFaWmxwDHqqYQnxorr+KG14EZbaiyKPqaqHUu+hbyOXtFcHfbQpQl02CCPAUkTneTU3z+EQqmgMXC8xvzUAh668x489tBD6Bvsx1fe93eu/85Gu+hxCbeIim7m3yqgIU4+66XIlSq4c3o7XvXyy9FXqOCmG36CTjaDe2tTmFiYwkJ1CUnU1LNVin06P2igUtZz54KcKQAPbK5VUa0t6dACYhWe/MKAUCdq8339Ayb4/YKXIOmJWLVnl928+6k3g+IDfOTrX8KOfVNYYhM/o/OGjfwuVUpIW21886PvWw4endYbVSrFI/ffaV2jYYDhwiCWwggP7d6N+3ftA6e9WD5uQ5DIfy+VCAtnNJmKJj5fsgHLImW6IUd8vU6iEiOVymzRr6ZDaDqIjUenQDz/j/dLS6Hed3fsyMLCnH6m1WAA55s0+R4e1yZ2TmQmv6/cZ0WifF6t2SPFPE47chPWFAjqOJaP8n8P2bq9n6Z40jlXIFcawKONaVx26aX49fd+gioifPeeW7Bv9x4020ZWpZvUHB1X32DbOT9P5wNx+geha83+56idpmYOCH3V8CgrK9OtqavIC753Vy6nKlbrPfBrP1oRgEen9uKr3/sBduzYY5F1DC1UpVREI47w7fdfi4JGoi9/+c979IE/ycT+6qGHMKHZM/TpHbFMleY5/0QjQ65dsdBnlOwMO3nKBssqYjWfyvr7gU0P2YxtDsKzur6iXYNzaX2kyc70coPZWbBkFBV0BIv8uwNFOFmDMDXblnTEaLVuWLhmJLlBDBqz2gKZBfTJlXweh60exbFrVqLAw/6kOZbOMoA97vRLMTK2FvfM7MSHrrsO1/3j+/GlX/0YtWZDKHwjsvI3mU1SRTe7lm3q/L2OSHcDE2z2OQcgG3pJ39/f168z6Q2Asna2ZcH7kqXPT33x/8+jvP1KpMKtA+CaT38Ke3btpeHRTbTqdRtRlglx1MEH4QNXXWlND1phnuGQw9bJCXzlxp+iqeF/Hevf1rFlxqnTgmesLas6vyDghydcqFhCwZfLNoudqKF65G2gAdeVAmabcRe75sGDPNpEwjZrQ76g+eHlXj3l+SFkJvmz74ilC+Ln8h54f7wWByl3hxvFdlIlf6fqFzLa/DwpQlF8QgIErVAWmw8aw6lrV2GIz1EM0LfqRJxw8tn4rx33497f3or8oavQzmawZ99eo7g166jyUEhWNDXg0CZue1STsuY9ERX1ZW9aAI6Cp1vSc/oBlAzAKfyuqfeIneOieTLhfrNJnML65gCvv2EnxTv/9bOYX1jA7CzPRcloECJbq3gWXV9fP77y3ncgdLXoWpDBh7/2VdQ4NiUb6oiQYp6dtBS0+T0yham97FtX0NbuoJ9DgrKmvS3Oi1NbtO1gTXB2x4F6mhf9Hx9SftpNxTTiAidulG0sunwfq3vmq42Ry7P1LD6Ym511J1waLz+roo65EgqFFoAADg/3NdNvk78ZTXOEO6d1G1hlYA/LKszzmYszRz9qzTqcccTxeMa5z8Efdj+EY9cdii/9/scKPHfuG5eb4eeIE9COxGWk4EV2FW3dOo/ov2klaUH4HDq/p5BDP1FOziEin4BuK3KnZfYKXubCC77Ht/cGdDJSPTVzL/x//+1NuPnuO7F376QO/SHPnmANtY+jxZ9x+ql4yYXn4+a778FP7r5LTY8WgNnid32tZ+BqegPPb8/qYfg1Nz+HFStW6Pw5G49mw5asvNvRYpG5qwEA7nwZ1eXdDHrz3bQgoYY38ShuGzHuJli6oNAPHKBPlabHHeXMS9Vqd3gSNwCFwvIsn4MFG97nAlubq1U7FoSVNzfixRNMbWRMoHHnNKp8xv7KIC48/VyklTwuOP0sfPOOG/HE9m1CKcW2nZ1HvVF3/YghWi2jsrE3kW5LVDNOJGvUVSuxCdaWnjZ9+uh6+voqA0a+3E/wPbTh/yuo289fU1vCEFd/4iNYWKhpGjUVkBOyeAulgQEcvPFgXHjaSfjp7XeI8EfByyfnKNiiLkchtohLZ0JVzTS/3REofSbAYI+WwOY4WRrlhwaYZtu5NLxml11K4Wv+KwVIjbWAVZ29jrTou2jNh7puWneqhI/CuxbB8d1keplpMDPgKRsayWra1p3ooTMAjEfohyiYh7comxuBFUaCUayzX/6Cv8SetIaZ+TnxG7Zu3ar8XE0scYLq3LxNv2KwFxEws1OuRGyRGyNPYXkursrD6mewdjVuECrGsuD/jDpki9OFcntKH12hH3CI3ds/+0k0GhGmpucVPTZqNtRIc2Q3HaJhwjR/vDGdZknBMmcv8EhR81MUCjXMTmCsKHCisBgQSUhu5IiaHbN8COIFLX2n2aW7oK/lG1ivl58OQplgnbjhzJ4f70n3wSDJV+Z4v0pFdUJH3tqomVE4lyKAhNTuXM4CLlLIXYaijdeBzDADRDJ2+Dn8PSNsfbabK8DTJ7wbsvGwsY5Uo5AGDlqJJ537FGzfuk2pGcvNtCzjeyeQNFpoVGvabETl+Kw8a0mhk07T4vApy9U968jGwtrBg1AtweXxCmj8cVVdyrCDGLuTMRzdYZmdIF/TuzE+8fWvYNvEBKrVprB7Tmmy82dC9K8YxvCYnaXOPFrRdKXs8GRrCOC1Cjx1SVagoKofTaHamkJju1aKRQmRm4BmmMGUmgl0Ph5HtFD4oSJdHlIoQTnrQAvgF0QWhgER74dkkBxHtFkwyCyDGtls8v1sTc7oc9hDoPo5aeWlopWRHW9QAx8IALmxo1xs/seBDxQar6l5QI48yvunm2H0L1eSy8taaAN0Yqw6ZB2m5+ew9uB1WGpaUBrX21iam0dSb2tsvHx+HOu93IA2JdQsmT/3zub4s0GEOAnn+TuuwYP3/j61xTlghu2BPt6pucesZQ16ulb473sefwxf/vH31DI9OTGHQr6o1Ee48+AAVh98sB1Nmg3VDcoGDGq0zLNj4vB1FDoXRvmyNCpAlnVoQqSOOSvf6o48UWzSPQrMDiCgNjJgZDWQfycSSC1TuYSU8EpFAxa0UI4M4vv7/WYmMEQLQjfB82vM1Gd1xKgd48n4wE6I4t8NCzALofiGpedm0xpINIPVrAFfTyvjLSqxczWNJrZxma61kxiHHnOEaF08XbJEhm0mr3N2o0ZLhwtatZAwuKdpG+1a13Xt0lZwshGwJjNXabz/7t9Zde4AjfcVq16N9ibeC/9AwXOo39s+8SE0mxEWF8m1ywp21TSMXBajBx2E0dFRTM1OyXxT+NTu4eFhV+hIBXuWSzbtsdJX0QBFLThLkO7kDC8gj35ZfMB0y7c5G8uFAxm8hov5oxOiLGswHpoFexFTsB5yKV/L+6vWaoKhFQsw/qDbopVgOhVzWBOjbaNPSQDq+TOmLgtWtAIUsqhSOm/Oavn6HV2PQxap8Uz1CELxWjOTU+gbHtIZczT9tbkFJM0I84uLQv40ccMxj72LcmLt1hv8rF/rVvIbgefsulnB9931X5pzR43vFayn/nZ/2fPDMqazHAf4zfC2f/4Y6jXOrKPW0RTxBApCjQkqgwMYW7VSJowaNzDQj3KlpIhVJyGHduKjR/WGhgal+eaKLKf2zQKeI0cky1MmqWl2HLdZCk260vwkoiuWHtq1fHRv8YGVNN0UrU6Mpbrl8JoL70AeDwFzc/HavE9/eII0iqddOl9NzNxo2NY7wOfz2D/vheZd13Puocv3Szgh0/n+OMYSz5yhu8uRjt5Gp2F8Bs3+cz32XHc9k6/xusppnLBAQ9DGjZ3pys8Njrr3Tzd3Bd+bpv1fgveVp672uw/+xNe/im3je9FuJViYZ4pT1BgzPiyPHx0ZW4EWz1UNM+Kr0ReroNOJugQNLqhP88zk53XiIjeLD4i48GZuE12b16FGWquz5eMKLFmo0Gxao3Ornq2UyooXFA4hT9LH5LPJSyfzRXPeeVaeTZ82KNfq3/LVDgWTmddxIxaUskjDz5J7IP2cfATm7AUSSjtyORQmT6xmcEaloPnX3D926XJjRG1Zvdm5eRFccwULUvkZjG98u7lMfc9Erl4l9WCZZh264FOm3R2lEtx3501/jsk6qEGvO+Dsdf27p8nwwL/fct+f8L1f/grNRlvCTHQSFGfR1+RnVq5eheHhEdGFS5Ui+ocGFeRRmymkpXpdUCwBlmqVg48NauTf+BrCrjqpmUOVNJ3aOPq95t80gEMMbCqXMSoM6vRQrVqdecx52w4r5rU85GuZQYQGMXIaAyJ7boQqwR9r6ba5fPzZ+2w+o9c+Rur8PWuVokS56ZtKK4k3MHhsNPRMrD5SOAzWuGGZxtWjJtrVpgpdeY0zIx7h5v8fkE15gft2NNERPMXKtZmL2+i+ZAn+J8FbU9//LvgDTQzR3XaY4m0f/QjaLaZACRYXaoJZmWpRUwZHhvXf+Pi4dn+pr4SRlWMStARcLGjB+DN/x8XwttyEb5G3bwsiBs28lILSyVGJ+V47KcOdwuQHIzmki8+loNH7Sofbe3/pDyrQcARC0pEBONwYLHeaqY9ccOioVu6wQglQgRpLp20dHMQgtMh6gMiFlvdzTDsF7wEm4QFRpBm+5CJG1RrWj41hvLooZJM8em5A9e/tJ0TDOnRWgM4vW+4eNsKHa6QgZtAF51IE997xn1aW9RvCHxLYE+Xv5+cFCu2/KbzPd7w+XP1PHxNyR3Ig/X3o2oxo+mmSy30VbQI+RK6YR2WoH6NjY1Ys6aKCnIJdslTLmUlh9K7rlg/P3zP9k5+LLWgSvu9MGzWLx6eyscOKIkaNtrZmi/7FPA1tdoyCMoEthuVz09Gy8JHVu8+TJxrN5dxex4rbgctadDcPT2NgOQeIm4NTudsRSoWi3BTNuoE+BiX7moHO8AlYX8igWmvg3GOOx9bHHkGLlb/hUUxWF9BkZuHaprgpmSlYCuomePAZVX20MSuaKJY4i6nYwUrYstJe8N1u1P9D8JYO7F+qPbCO8++33Iwbf3eLmB6cwVpvttRMuUTggSzb4WFpACtffYMDyBazGBoelpA0BsydskBSJk210jidHr188iMbH0mioKnnmTpK2RxWrTyWgosiuQsiiL5TlwvF8WFWvDEXwE0gi9ED7XKz80RMjVmlptPXu0FNis79MaQy5cu8dS2uAB/bZEL15hYUh2iKSKGoZ6LF8CdcEtvn9TIF+vkYm9eMYSxbxrZdu6U8737b2/CO970fLUcKFQGTpedSHpe/+FLsG9+nieIkYDTbCRaqDdQ7MaqLiwbwaPCT9fzbKBEneEvnTK99D1ovAbFX4/k6f0Cu9+8HCp6HF73tIx9EQ1BigrbTiqjVUV5PXj2FTAtAXln/cJ+IGMLdXQ+4hv0zHaLQchbNKzjiyRAO4aMrkOnvOe+eu52WhP6W9Wqhda58aahcRr/XEaU8Lk3om1kw/T3DyZvU5Mjyap2k6Q4Tcpi+LI8zb0a/srly1GZtnhangwxi5042ctiMAB99cxPpYAaetunm5pn1KiCfy+Ctf/VaHH/EGlz7/z6I6blFNYf84js34PmXX4HxxUWlnzwHgHLaeMgqvPkNV1j/gPy6I7XyKIG2O0/HWciY6SspaHrUAMG9t/0qVSDUtfUuRXP+vSfH685e9b7/QMH7rIAb4+d/+D1+cvNvEUWphh00G0SnClocbjyadZqrQl8RpQFjklCQtBIM3vh3wrvM8ZmG+d8pv9cJGHbwMXc19yyHJnJDETvQfdCMavKGQZTyvZq358azuZRMGAPsaFW6CnXwdlujWfHj2H07811CdHiBdx3i2jEbaJpm0XJUFxbtaBN37h7TNm4QnW1HbN5lE9xkwgYyWYxWivjsR9+PsFNHOw7wzre/B03Xa/jlz3waL3nNlWh3mE1YZsHPf8HzzsUZZ5ze03NvG2B54ANPgmSvH/sarC5BjZflvOePFLztIPtyw/APTODdMZm9Qtfe2a/pwjj3PId23/g4PvGd7+pExHbckuAzjvLL06ZKRUP1hsaGke8rOnDFJmPzxpka0ZTTRZDRQj/JtI9HinNx5+dnBaHq9GWNPOF4VAI9OSFryvmzLO8yFfIgi82zITQqGNMFYvRc3ADcVLQAOvzXCZpuh75eR5u61Mn/TTUBx6admZ7pNjsYNsSAyyJ6uQimkJrQGQu4oiWjpVLzZbkfV5x/Fs6++BkIkizGJ/bhwx/6FBqMUfJ5vPTi5+Az//YdTdu01JDQc4APf+BqHd7EjmGnx12peSU0hWZgZ6VkUdoJtd/1+/9Ig2yha+o9r/5Auavo3zPHpTeN86aef6/Xq7pxfsjMUgOf/eEPVEsnlEmTT1x5lpMeuLitNjYduQUxazOu24MPRvNMn7V61SqlQdZTl2JgcEAIILVJp11ns1Z3dnwyXkSMWB5w3NVuRvochpix4z1d5G8Rrx18SOaFnbbp/L3O77RN7eff2IGExmSlv6fAVZRhwFZj14vx5ClwKYeCNxZebB4A/y03ALqrorQ8aEXIxsDo8BCe/8wzcfYzztPnXv+5L+G+ex9WF8xJxx+HxflF3PfYE66WwbMA2FxBwb9dNQwDgNxhB85S+yhMrogNopyOqfpEwXoO7rzphympyl00rqeTpjdt6BX8gZvCd4dw0hU1MQjtSBKal0/827cwtchTlFM0eVhRjuYt0YwXYs4Do0PYfMzhOqyI5lY+OZNRNWtsbMxKmSREzMyocEJzPjQ4iGLZXIUQOmnB/1fXm4DXfVbnvmtrS1vS1jxbnk0SOwOQwKEUuKec9gKnvbSXnsDtgdIUCJlnZ3A8xU7ixHYcGw+Z54lACCWkgRAgKVOB3lKmACEOGZx4HiRrnqWtfZ/fu761pdLnKk8e29LW3v////u+NbzrXe9C7stROh91Op7akJ1nLyRufEK/EykURSYVaURXnpFb8TTVo3zNmmCxEzAD7Ispl0zrrC7bkr0UvW7a0UK+IDgmsIbrYx481cLJoVHNigXIaW1stL/7vz5g7/3QX+geb7h+kx3vHlDf28qrr7aHHnzU3jx8xOlgVVXeJVyWsS2bV880Y85C7sTO+aPxa6E9MB0Azn+88LViZUN9iRY1G7HTwiew4D9tgj9e+cK0jYwO2ugINelxEf1cLqzCKusb7Ma77rGRsYIvvAK4aeuht34YgGTalp5xmoIh0Z1SHqqyLHRgTnN5ue19Y4+iZ1JBkDayALILXACBovrsRSzk9PrJ5k/eh0UQ2WIKfzzuQzAEAVeImSq/m8gbs0UXtVlIocYnrKWp2V7ZvVufB/jC6zWpuTTOnM3lAZUC1ERGrhD6Q3iXtYs/+yn78/f/iZ1z3lU2ylBirFxFhc1ra7G//av/0973Fx/Q765ccYMNDY1YRVW53XfHbXbeZVfa0PC4VWRJbSutOldtJ5+yxD591pkl9ywnrTx9RrHbvzczrox/w2FUeZuFr6irNQTw3E/8UZVuloz4fzH/kgKdtqGhfhvo7xHPjxMERCqQhViiaLbveJ89/Mx3bISceBoR43IbGhq1wd4BASInnn6KbxLkT5P6BOkPp5vFZNwZlGA4dt7hWnDWa6qzK3VT/bxCD9JFk7xQwmvUyiWSoSNaIHikaSq2AMeGzm7i2zvxwjti8bGHDx6SLw5M3a2fa8fOPumeGkZ5jFSuYOUVVXbRP37CPvahP7OxiTErL5bbhZessr7hwVJ9YF5Ls33yzI/a6e97l+bW3rr5DkG5bXPabOXyK+zK1dfZ1DT0NLIbh68/9ekzbemyJQmjjyFFDmyJZJkImRGTKRZTvJEKPL/8wVPFLHZfKdLMFzcwG579r7Ges1X7+o7bYH+fHkplzjFx57MnHRp2fzZjX//Bv9mLr79pY1PTIhYAWHQf6xad6MTTTlYO63VkR76Ae0XWmPaBQSwmChQUPKj4IaoEDWtyKs1uhWyQkCtRq9Vc4eVZOPgEU4Jkqd2X/LMDO0Q+QtuS/JlX2aZtoLfX5+6Me8SuOCBlDWqc1Ewel0VNp0YPlrEs+N6Vl11s/8cZp2mEKcdb6Np0mV142TXWOzis3ye1nN/eah//xF/bO05/p3372y/Yt771gjbF5ZddKM7ffQ89rnurylVZZXpOGzauKrVuz14b71FMGH6pVO3Bu+TZo9bw6399ugi6U54oxrFDSsWXPwJrwnxwUnqPd1tvbxf9jG7yknBh7K5Ib8SRs6Ld9rVvWtfggE1OeH38eNdxGx0ascVLT7BslUt0ccpFhkgsGnrU5CpFnypo2iVpFyYPd1JV7SPNggZFCkX0r0pdRc5pT4gsTnoBRpG5pmI6HKsKmrphnLbE7/Ue7ylV8XwGruvc6jDHeLGEoP2xKW1rqLV7d+2Q8jUz4tHpY2hh7A0sziWXr7KB4RFt3urKSmtvbbKPf/yjtuzUU2zTplutu3tAz2DjxnX2nef+xb79wve9M9bKpAmAZbxhw7ViA8emi8XWus2ur6TFn12QUVT/mx8/W8RsVtbVKZUKzvz/38ILiJiatKPHDtrxrmMOqGRhq4xbQ0OdR76iKGdUYXLyAtQp2LRlduODjwsRm6bXbmJK7wG/bu7bFjijNlPmkxdzHs0L8k1Yusw2hY8xoN5Kfb+6psZPU6RsjAdPzRK4GRZN8irqn/NNhO93yNZzfRDCgwcPeaahnzlHLZqrQwtIFbIUs0mnz/XX5RLmtLfZI7t2WFkmFW2o7lERTGij3KgqekW7YvkK6x+gszhj+YpKa21ttE984n/Zyacus3XrblR9o6q6zG7eeKNtu/V2e/XNvUpr2bCtrc1WXpGxdetXKo2L9Yrhi1E/iawrFrw0MQPYmcD3Nz95tshfsvnqmVGUs4oAsxUewhocPLDXBgd7rRZeO4CLUgLUJp3gr6JBSnV4qAzrpazJDp/IVtj6ux+08XEXIOrp6rburi72bhpGAAAgAElEQVQ75R2nWi5fJVpWTIuWdEcmK5WpoBITsU6NjothorKsumYq1FnDahJjSAOHiD0hhsQhWqRUL1eRZXLCTl12sv3+dy/p+zBo8dke3KWWyoT5RwnWT1XS403ZwalvW2wb1q6yGvAHZt8orYJXMCZ9v/8SBxeKduXVq6y/f0TpcS6btY62Vvvfn/yELT5hia1be4Ng7o//Px+z//7f/9SuX7fZDnV1C/cA76+rr7X/9t9Ot7/+m//pZUNflFKNI1SqWWjJzKT0TsLb9CUmjoIWXpEqIkJqNPgjiYlQdhbiNWl73nzd8hUAAVM6QbW1TIScLFXUWCzMLQ8eU6uHKdpUQWaNhzc2VbRVdz8iXzvQP2DDA4MKZIBvS0UWsPKJcUX2oH20PQnmRA8Gf54ia95P/w5lZvXDe4Qr3ZuE2omQmS3X3Ly+48fVri3oGWsSfjHQykRsEOkyNWzoz1Te5Tc+eebH7NOf+JiVic8fEqN+qpW3o10z2F9iNpWCQCvaimuusy4NcCK9q7B58+fY587+jO154y372teeUoFn545bRL9esXK9DQyOKACtq6nS2Jfzzj/b5syZ4zUTLdfMBogTrhOffhLiNbGh9TMWXgUH8B3pw/6RyH+KfNlBv3/pRWtpbVSwg4hIZUWVFgUkiTcLnhxBhEqjqp5VauFFa05pVKE4YdduvNsK9XWS7oSQSLfI0tNOSRRh5qP5o4oqXq7CdXNQfFQzQUrB4kaD9IirCN9NLd+LKR5TkB3wRZzgNKqssgmdBsq0iaemVm91nrjlkD0rFq2hps5uXLfWTjnxBCtOjNjE6JBNF9OoD6EiaeEpKKmBdEjmPsy8HnwmY2vW3mgHDxyVqa+qyFnHnFY755yz7Stf+arteeNNETm33rpBa3HJZVfbRKGo3L+utloLf926Vcm3J1WwpK9TMu+zOIhR7ZRf5z+58wzI3bNF/Bw0qap8zQwpD3CCFl8gycKk/fxnP7Y6nW5Mablm0kRtOJgutAHzoNVpGukDTQnw4NOAez3MwqRduXqrldXUWqEmp46b0aFRW3jCPB/Gm6pPXjIlGnWFKZogRGAYGxcaqNl3IVGCWeUI0cQwNq7UjxPeP9Dv7ohWbIE1nutrkzKIIE3OUPqTpETGoSinqdMANR9835/amiuvtPKi2ah634gbmLfjA5SC2RMBltDHXKWNDg1IRzdcJDgF6eimzV+wPa/vLZWYO+e027nnnmO7du6yvoERe9/732Wf+ew/2NDAiF199RoJOWBl6eVrbKy19etWWyEdDA9WnV41m41DZ66upyQL7ylfVCW18DwsdGkrq/PqWg2TwALRqPevP3zB5s1p18PioSslKjI9sqYEYPBv0LMQHyZ6la4MHHSkRRPY4cWNgl25ZqsNDY7ZZFJT/qu//JDt3vOGjQGkZKkbx8hxCi4geUNC0UT2EE3Z+XlAoZxexpqqmRLqUlKB4JRE+TR2vrc3BZ07DQtOOS9WT8BMgXbirJ115sftr//yz60yBAJxIakEy3Pxh+sNlVrcVOjigQPYTIwjYDaDi0RN5LZd99qvf/Vb/QYWcV7nHDv/gvNs88bNNjw2affct0uiDj/50U/t4UeeUNBLCkxgh4u9Yf0am549blWAES4v9QSIfTNLVj3a2tN8HFkGsHr+AnyKOSwkCQlFvoUJ+97zz9mC+XNLrUPUkTkdBG38Hg/K25jSlIbkU928uYq0s2UyOoFu7op2+bWbbHQUwWL3ids3X2vNjY32Vtcxu/OpbynIms4SKnncgUw65n1oYKjkNnhw1No5wQgmkwpiobzWjXIkMLzntJ4ZzPhgXTPbSySGgk1PeD0cw/+h95xhl1580cwpUtk+gTZJf4aYQSdM/p0W7TQYSBOoIVKaDfb3ei1cQaHzCCnFPvTQl+0nP/2Zfrc6l7M5nW32sb/9qN1//6M2VZi0u+7eqef58EOP249/8gvLVVWoXeqEE5fYqacttb/6q494FlOqqDocoRi7VF53/19q2UoFptikmV/99FktfCg1lFUjLwKJYdx+8MIL9rYl80oX7sAIxREP1hzzpuqWFpRJjZU0BjjJMVIfZ8b61CQPmKbsipWbbWh4TH6Mn9+983qr1M8mbaJQbhseecSmilkrpJ1LkYeawMjQqDN3ktwqAaLy81SM8I5ZFzwQ8yY0bpPbIOAsFZhgoKZIHez702eeaZ/827+xbMYBHW3eWXNrg7vnTYre8oQLCVPuuZUTPMrLM5rS4dCtT5f2RSmzJ77ydXv+hR/q3/nKKmtorLWLLj7brr9hs7W3t9qKa5dbTU2t7dh+u/3htf0im1SUZWzBwnl24UXnys/roCVwYAY2jgifR12wF1980d71rneVXIBboqQfHAuPaNAogVoNufekff/57+gimhpqZ/htSXXaETAvd0bO7IvvBZAwO5xULyrgGjwAVTm0vNwuu+Ym0Ydj4W/ftlYkTtiuba2tiop3fPmf7EAv4gRaAu3eqfEp61HBxrn0sF2EUSeeuQKxSCeT4qNOoEy8/8y7TxBKKLdcJmNn/93H7S//x59bVZXz54Xvp8jeEb0Z90c2EbFCtGPF5lIRKfUE4ttHhocS3Suwe8fSv/P8D+3Jrz5dGsXe3tZqly0/Rw0mdO+wyeEu7Npxjx093qvnVYuSRUOtrb3u2pIiJsGoW9YY5SJH6qQP/kucwzj1EeknU/+sOmlYNAYHEUA9/fRTdvLJJ+qGCXLYcW6yEidb0bJDnDxQmbBZYzuFf6dxozHvPRZDQVW2wi5cfr0NDbvCJH7ujm3rhANUotGiuyGarrSf/eFl+9Lz38O5+jUUnWHTfeyYn6BUD4/F8YDQF1dky5ioHLku+IKZzW9pspvWrLD2+nrvLk26PCI6pA5dPcA0GCk2gOP4bvaDCqZzLDVtmh99mANZiluWJJU+i7j6rz/9ud13/yMKRCGcNNbX2YpVl1p1dXQQZ8VfuG7NRhseG9ZmbKqrs6rqClu95pq0FgCSKY1TQhGMx1my6SVqmd8Hr9GhpUnzVz/9pky92o6GR+0H33vBFi5aIOozJru+Nu+88SLFjBk834WC3SRi1nkgihjl99ko3sHhgVROKZiozsCvmaxdsXJTCthM379n140qENH/Hu9DuZQHN5HJ2LV33O8AROo2IVXr6+3zjtxEeIgALiJcFt55Zj6bDbPN6Xpww3orKxu3wnSZGD+FIqVTb2TgofC8iBf4S2QE/AnCCWLnnD6PH/izpImfNOZgzzJwwQcl+eKE/Dob9Pe799jNm7eKOs4haG5usFWrL1fU7uaYg2V21fLrQEv0LNubm62uIW9nn/0PrgyKi0nxS3AHFUeAxaSNHHN3JLUOd5/ANU3+yPzyJ98octqBQr/1jaftnW8/Tdx1ghcWlO+HooKCiRTQOfFgZgge9fN5nXOVdsUpd7NeUSJMRmcKC3Xt2lu18Fw8alcP3rlRHHTyScAKoU78fuqfw7Uc7h22TffdZ4VMJbwTmxgfs5HjA15jV+UpzVwTugbxg66TolVDy8rmbH5tld26eb3oymEVwjopABRVimmODkBxjqJZg00nV5WYupoNk1IltzJZUchp1BSSmBpK/1OKpdebdR/rtWvW3KgaAYgc+fkN66+xyrx3DWsDT2ftokuvVhNmLpe1zvZWe/s7ltlf/MWf6RoEa6eqYty74whpzFnqsIkMzWv0qbmCLODn//rPRdifzz33rC07cYnVVNFYjyKEY+Z6gCB7oi27VruQqfSQ9drU5kSlie+7frw//JK/LRSsurrGwZVCwVasuUUiAgA1oH93blsnwqWbZg+c5NNTuTWTqbCqykSxKmZscHTSrrt5i40VfIePFt0X47OrMlmbP7fT1lxxvvD3J/7pafvO935gnS0tduut14t4ETlt+HK5nOq8TjUBGqdYFLCkJOHjv5JJTaFxIHv6fHoBFAzGwMQU1AmrD1DMad0T41N24WUrFOzyzBoaau2mDSstW5Hg4qLZm2/ut1u27rKKcsx/xpYsmGvLr7rEMpmC1iWYxbMnRUe6GJM9ZMmTJaahItyhNuxPn3+8+N3vvmCnnbo0MTxc4iNStWC3KlKW6pQL7Qgpc/6+m0janBOYQt+7QI00CpTXw58bEUyK6obZVWtvsf6BARVramvydt8dN2vufHkGnRifkEzs4PPnvDrn4zNnePQrV9xcaoxQWiWt16w1NtZZ59x2u+DCz+l7Tz3zHXvyqW/a/JZ6u+ULG8UbCHMoM5w2gqJvYbyJmyC1rcSizbqbixgioiosgtqjmQ+LsGAqAPlrneipDt00akVoopXZ2ede5oTMigprqK22LRuvs0yFxyZsqPvvfcx+8eJLum9g3faOZlu9ZoW08pIivehlIe8+E8DGjJ/AFhJHIG3agLgzG1aeXWxrb5NClSSzcg5IBMghdAzfLUDGNdD53ynGng55O5J3YuLPKQQoDYLsQJ1elkOgsDdNTE/blas3W08veDX4ed7u2L5edfuKLPECVsSDLKjOcdpwG8C/nmZlbPW1G0Wj1olSX7gLLpRnM7bkhAX2+c//g0zwd773Y3v4sSdtYWujrb95re41uGhebk3zWCPVic2VzL3nhCYNHv6OSS8FkOL50biAOINvmBIXY1ZziJtc6U1bMVNuZ597qTpmWNimurxt3XKDwciLrGjjTVtt3yFK3rRHl6mCt/a6lYp5mPghYCqGKSWmUaSVgqFnz6FN4JIsgdZryjIP3bamKJECpj4nJQf0UllwuO1cMN9n8UhznNPuu4jXxIWGuY/GhdmuwLMGtxLezZq1q1Zvse6efvW7N9fX2q6dN8qiUL/WZ03RxeradVLByniaKECoSGlx1G6+eZf14S6IVBWJ5xQYMQh44aK59pnPfkp0rkNHj9rv//CGnXbyMlu0uFN0anrl8MVsJty2UjivcWrhnPvuZVUWLJfzThgBPtqYbr4DyOHa3D07WBVBb4xOdTTZlbimy8rt3PMut1GqotmsNdbl7datN6q8LZ6AmV276iYbHByWBauryduczla78qpLne8fbVJp4UMggusrtYZhOXhuCUAS6kmwGdnFU49uKfJwpJScfGz4AoEwqTpFJEmRI3xiFEViZ4m6m7a6pLaS6A+vj4fA+7LBeGRXrtxkXT39+vu8jlbbtPFa3xjlDiCRiaoZMgkjwWzJV6NQ6WkJVmPj5tutq+t4+r0Ka2ioFyO1sanOOjpa7JOfOlNmloCLY4I1IXLOZXMCmlLeWLIirpU341pYBLF1vX6XXh8m3Is30eEzG0SLDRB6dv4MQ8QYQnTWLrz4KhtJHT51+UrbsWOTwKuQTrl6xY02xgiVsqzV19baR/7nn9uHPvxBT1Ol7emB9ezgkc/l50o92ZRcO+4mYfmy1jFo6smHNxWJ3Gvzdd6tAsslpSu6UwV6iOL693kQ0XzAQkTBgw8jOnfzk1QhJj3FC2mxMEGUVq9dt8WOdPWqy2XJwg5bv+Yq158LkaCCYwFkCyx+c2tLqWMmINC77njE9uzZ50ui4MXZMvnqnL3thIX2d5/8XzpR6MjA2OEhEUVzeh2EcuuFC/NbTQydNILUv+dMW9+MiC0kD6vx5kkpOymGJ6hA7ztTxp0hiWCqBABZwS6/Yr1TyOAVVOZs584bS5ItLOoFF6+wTJlr9rQ21tt1668pSbUQJM1G61iTCLi5ZpWpIYKAaqaRrtRdWAusreKsrzy0qYhpAjiRZKeK9y4XonRMunBJICDVvLEQ6lWnUpceXpjxvr4+q63NJ/66CRCKFEUdKdPTlq+qtKvXbLajiCRZxk5/x1LbeMNqO9blFGJF3DKvvjC4ABSZS+yeJIT81a88a7/4+a89709SnpA9GmvzMvX/++99DjubmSAM8851VlfVyE3lESdOSKMTKWPIQFK5VueJ067ollUDBUp1Sh+9UMXChPXDlJcoVknXPho6FOJp6GLGJqen7LLL19nwiAsmsJluv32jmEK8fnh4zK5ZeaO6Xri+jpZmW37VBdbYWJ+yJdq93QLp2SSOXUi6qlsoiUXF4k9Oem2hIFZQ0TLPPLHTYf3EEC09iFS/hdzoJ9bLmhL2Gxv3CY4CRvyUicqcfocLUJBFPp6CDPHjk3+hpLnu5tusq3vArDhuH/nIB+3sf/h76bROTjnOz0KJbDmbNJneV71ykwX70Q//zb713A9SC5F5kakwaTVVNbZkcYedfe5ZJb8dUzV0ipl7kNqQfAqVjLPex/vrPHMQbSyJL+kBaayIl6rDWkARE7CUBhGT+noeP0Nr1sZELpyYARZxttwuv+I6G8CHp8aQ23deL3CKNHLfgWO2+dbbdVX8bltrk61bd40GNrAxSB1j7h4Qt0u4eWVR1PJZqXb4eFwkhJviNHqAE5b55y/vKEpdKqlO8QbSR2WokJoVsq7QkM+rqUDyImmjBEZNYKWO0tR2hAsI9E3pA/1psQkSiLFq3a12+FiflZcV7NzzPmMf/NM/MXYlpd1SO1OKntX/HsP1Un9aVWXefvbvv7SvPPmML1sCLthnNZV5W7yo3c694LM2gFxYdbV67Fx0AMq2F410f0HhKqlJO3PWeXze9qTYJQ0+ZuEduHLLhDXxTCe1Zycp2IgVPNjDiqYp2slDL79yvQJTMY4yGXv04S/YxCgzP8yefe5f7BvPfV/3xeZfvGiBnXvO3wvoYWGVVeF6RVObae2KjVLadLq+mfmBauWachmXzDNP7tJ9STSf+6P5AHpUak3izSXMM6szQ3LiibvNRXDS/cykScVRjEmSXlgETqmiYtKJyQnbcMtdduhIt0zW+uuusCXz5uk9AJMUF9Q4kBTyJ3yPVqXmlhaJKtRW5+3F37xsDz/6pCYS4YmVhmbM8tWVtnjRXDv/ws9pEfF3LDqxjNIwtRNFFO4+XlIkImqSK3ljI6cJV0Yc4q1UTufyeAewKXHVWeyyjDZXTY2TUBzV45ky9mw2G9aVsq66+gY7drxHz5Hq0UP3bnFpNdi1W3bZwf2HBSXn8zn7m49+2P7sgx/QhA8xmypcFSwieFqp9T4zd1WCk9lwMUJFC53EETL//JVdRS+0ZA3/jE9nN4cEiSDNFO0TaHHyWTy1IScqNLtesqOSFnXmZwnqTREP5ghUTOlexuy6m3bZocNdetB33r7ZMgValLPSveXhYvKxHIj3ElOw87kWsgvy6FxFue3dd8juuONhMVcjd6anLJ+vtPlz2+wfP/spvScPRi3XqeUZEMjTTp9Dq02dsIMo7tCdwzw4ZStpfrteA0aRhvTOLnzAk/PBQNTlgZvDgzoJNMxvIgnZqlUbNe81AuqH7tta6nK94sr1nl4WM1ZTW2nXrb7GqvMMJUjCy5p26WNbWUzkY4LVzLrwjAKMinm6cnFYsDQFK/PNf7pLZd3x0RHh7J0dc7SoAcWyMCxqgPwK4ngoY+jI5RxXTjVn2C+8nofKe0SKp0i7psb6epHppJW5zDZsucv27ieYm7Z7d22x0VHXguVzaY863tWtMnFbe6tj0gUX7yNvlpVJzYq3bnvEo/FS9cuspjpnC+Z22OfPPat0+jhJdOnILKv44+6BgI2TpDRITSGkfIg4OOvWT6+3OuHyAgQhaJVaRsbUYRvQKe8fVObIhlIQUar9Y1k23LTd9h44oh9hrR6+f5sXfjIZu+SS1Z6wZZBmr7atW9bLGmDXBBOnnr3gAgwMuhvz4pLrB0iBi6JNqilEql1iCX376/cWCWIYBshDr6eBsqxMZkunOBEWuUBSIXwtUOv8BfPVBaN8PeXamobADhwaKvlOHrgmH/NwKirE3CG6WnfzLtu3H8Jh0e697RYbGOwRT46NEf1uLmrkSo35KsfxNWAHiLSsTDoyW7c/Unp4oZbFaxfOa7eLLz1P2EOASogQuniiq2ViNuvqanXvwdlHWw8zEOLE9Oi3d3R446OkQV0xm9erkjcrBhD1WzJrnh56U8esQFFyJCCgGbvzrkft57/6rbue4rRx4r3nLmMXXrhSXAGRMatz9oVbb/BYIJl0hiV7FuLWhdgLy8VnKT7JmA3098t60mAZBaUA0aTg8fSXdxRJCWCv8tBZIE5+Hb3n2awWW8EWQgac9sqcbhqzjWaqWogSpTp2VcmspGmVIUYUYANuZMuO++2NvfsE2Ny49nKrqnJFDCL+uXPnWm9vt/h9mHuiUTBqmgoamMhUkbPjfT3Syt207eFSJOtgDx0nRevsbLeLL/mcyq0jzMqh0saJ1agSBBRzSblaOtNKrSR/htCR3FZE9TktOm3bbAoWU0JNqUGzVPhI9GtMKbUGzC/uM0rWOqmSP4XoMWZfeuIb9qOf/ruXbqen7aEHtrklmyjapcvXlizVkiVzbMVVl800iRDHJFfiwxbR05mWRWVD8qxiQ7ju3ozsCwuuRhA+876dq4twzcnvhoaGdcNNzc06ZWwAgistSNJiV2SMhPew5/IaQq+pkS4jovp1ivypPGGuBQer6lXU6afosGn73bb3wCGhads2rrL6hjrr7e21fGVOFqOmNq9AL4KRfB5LwAiQvC8SsmeZrF2/8Z6S7lygisQQcNXPOedT/6mowoNtaW627u4ebQQWX0UgJMxSB02oWChQUq48Q1dSeprN6p7AFbAexD3yqakti4VXL37aOPLvCXbmT8Ajspenn/kXe/bbz/v7F6bt/vu2CBc43jVoN2zc7nX5TMbOOutMe/97353qFR6QBtaRiEkJeaSJM5uGFVBPcJcY/IzI+wPFyzz12Db9fn9vr8y6JjAg3znOhMcaO9bVJRlSpQCa4JzznF18cadWCRiQP0Hsl8DLBXOl9ZYqfT7IB7/j+ey22x+w/QeOyjzt2LTWxidHxbEnIg+aFO+Zr8qnaNwnV/GAWbDJKd/dW3Y85sIJjhK577aiLVzQaeedd1YJU/fqmJ8WeAEekfsQhND04b5C3YprwISWxpmkBRQ5RYOKvFAliXBhDQm/T/AoboUrIThlc7Q2Nycl7kptjH/53r/Z40885fWfqWm7686bREP/2X/81h770lNpgTN2w/oV1tpSn4gkXq8I0Cj8tQLKcDnJCmhRU2XQM4yUgUiZI2OZB3etLerBpeCovb1dN0KgI5Rpako36qXHENrznBRhQt6UBSDCZcE1hVGRI6ifpxj45SjiuBLkuH35q8/Y7lf32vve/z778J+9x6oqMtZY16AuU8zf8PCAhuqRaYj1guhPmhwtl0JaODFht+583KN1wff+8Cn0zJvbYuee849Q9EvmNkgkWB+v4nl/XnXeCzDE6ywms2DYqPj56LSJdEnVskSAkB+PPJ6MRhp7KHcXrLbOhxPFEEDh/lOTcplcx+4/7LG77nncpssgik7bPbdvsInRcXvya9+2X/92t1c1c1m7bftNNlmYSDAwFctE7kzgTqCGKhKBpSRsIhBV35z+O5HWsUkyD912XRHzLT+O8lQFPnFE9XNyeRoAJEeKxnxlpcuGxulJ/eE8DFA9ImF0aWQFCtOucjHpUqUsDnGBFC6nRq2vf8TaOxdY30CftTfVCFQhnqDsSO86Pp8ty4WrgVEzU53gqdoCM2anp+yW7V/0DpkUvbLwbLh5c1vtwgvOFo8vGLNcC58fU5s0OEnux+VRsVDcBxMmws9z35SbOT16JggQp4kVGvaX5MSoafDePAusppetedppmEHiDDJlA637w0d6bOftD9oU7RKT03b7jvVS6F69dpONT7lJrygv2vatN6R+f2/R5n0JgiNeioYJXi8cgdgs2Eiix3n9QdZ4zGf/lhY+UjcJC6RZK/yd00+jfnDleEgENvh+HiILSbDFG9bV15dwb3xgCPFhmicm0wAclXLZOFM2MubBGgFJU3OTTU2OiWpMoSYw+YgHuCmkTzipOvkEZpzOyQnbftvjdrynr+QTxQ0sy9rCBR12ySXnCgZmU3M/nFriEs19b2jQQ+F/dbjU1np9IbFWgEVZaH4Gd48NpbI0zBxqGmk2nvDxVP8Omhgug0AQcYM4iQR86v2bnNR99A0M2+atd4uUQaq665bVet+r19wiS8RXS0utrVtzpahXDh+7mw12b4A4ZCkREwQaCVfC3WKlN7Jq5NqsqdrPffUOVec4NQFfhnnG1LHzAUwI+PhApSipVs3rWfyYDs2Hs+gsGD8bGurTQ6mqIlAb14Ai3gPW7vAI05XGRSnm9zEenDhOPBRlqURD5EReTGM33GSz8SR4hFTY+Jjd++DX7fCRLl+wZOoJ+uZ2ttglF39eboVNiG4OqRnRb2AToYQp7kDykTz8GDEWuTndujR8Ks+vdNWNqJtjXsPPqwyaKnnyqXQRkTqlmrhKpQwsmJy0o929tnX7/TYOUlqctju2rpE41OobvpCGIJudddbH7U//5FTxECOg00ZKuLzirtR6Hd8PX88aB4jm2ZZDz7FBMvfvWF3kwXsfe4UEh/bu3VuqrXNC+CgX7Eecr0IkR+XmExMym1oYhuPy2oxDl/y7KhUrOHWcMjVCVFRYXUOj97mn2vHSk06yPa+9qt1Zm3dql5vgKQESwqaTADEwRvTb4wLuuvdLtnf/4cBIPPjJZmxOe6tdcP5nk0q1qzlSl48TyGIp2k4Vx4CTQ1YV7r6gaYIEPThXsI7R4qBqLL4zV71FWhi+mLVeB/DeA7cibOYgdvT199r4ZNHWb75H/Yll0wXbvmmVmiCu23CHW5NCwbZsWmkNDXnXmJ+loKl4JPl6ucLUnuYTrD2IizQzYgBxJmdRvDNPPri5qFku5eVKdfBv+HR8ReSyfIh058fGramxUZOeQwUa0p/06Kp9Hhw3J6nS2tpSJwkVM77UKl1drWIOvppNIOVo2rAy5s2WVJGkLJkGBwFiJFCH08r4Ut/97p+/+8L/az/6yb8nUoSbMtK5OR2ttnrVlUltclJsov6BvpIrkwImLqC83A4dPmxnnNp7wtEAACAASURBVHGG7d+/P20cFzyk946v0RGkWP1gEHuoOFNI/HQtEtVIL/mCZsIeHh52EAslbmfwuGz5wADACmXhCVt5/Q4bROuvttZWX3WehgJuuOU+cRd57Y5ta62y0q2Gl3T91AaHD0EJAl9POJ14QeMr68kaIBUzu1gWLl2bgRMvOHNyUmkbAR1ADr6NXYOf53TqgZaViTwQ/5bWfEKmODm8BwEOE3m8uodvn3bwowbhYpSsahXxk+ZJ7EjtVhU2PTGu08PvifWik+vTJAI0UmtSBbDujMn68b/92p57/kczJAaB4UXraGu2Sy75vD7PpUhclQq0TeBTZaUNj7hvx2+KXZvJqO88AlG+R8Ap8inFGXwmQ4/QpZ10N8hmlYpXb59iFhhZfhp9ALCSTJlnL37JGihtnLDBgSERSYDAW1oarLd/xB59/DkFfOUZAr4NUr8oSxp7bDanpSW9H03PxAV54ciD7jRRUi7HSTQ6uMz7FZTr5eLMfdtXleRRiBbZaSw8lTAwc0w/1TAV+4FjBweFZXMDkiVFA25iwos2lZVqbyIXl79XLd/noHkg4mpSfuK9i4SNxe4c6utRkIf16Dp2TA+VGKMhjSP3ua/MdEWe2xEoLPBrew7ZV772zRmdPh500ayjvcWuXH6BTtro6LATRhIW7s0gBUXz3G/QpOMABOIWFoyUTGmZ6tmetlIdYFOxpG45/MTTg8c3WVjPnRl4QDXPMx9VNUPjvrzcjh3rsjGJPUyoU+bbz/+HvfTSK/aRD73f3v3OU0QjYw1k/pNiFfcUMKxKsEm2XDSwtLDMo5UGf5KlgTIewZ024z3brlV1TunMLMIgb6CHklgoBDTHjh3TYvE/pp5Ai0XjxLCz0GZXBC1JFMAPj045FZ6XVgl1Q+mivqFBwAbvAZefzhOsA12vnqZHH56f+Gw5phKs3LONnj4Yuhl75fU99qXHv1k6WREftLe32PLLztECtLd1iIeeS+NJXRfeewTpVcM/e7nWI2fSWSwULof75+HREsU4NJ4JQR6bxxnIfqLk+niPSUaCIVPuvQUQKLkmCUgkBlBg5vw+vQVo93FwYNmyOZmRg0VkA7uCd073jJXSGqVpWQHKDDN5S82sHrkHTyAkVbFkfb390jQQykpQeN8XVhYx35yuzrlzZWZZdD6YD+MEYqoxf0TGXCw3HmYrAhHMF5EvEiOcJAKjU0492d58881SH93AgOf1gXpFqzVtUJXykc6yZUEEqkwVrLW1xWe0ChFz009f/sDQoBb7SHePPfjAP5U2bUT3bW3NdulFn1WRgnQHISbwcyhU1Arw+ceOHUkyKv4wdBKS+dRg4YTK8Z6cZMQQCSxZUdI9CjwgvnJxQ0OOeoIjqObgVCf+HXT1oHFFNsFocg5DSTE8658xMjik9+BZzu3stOPHfXgTh0ULCzO5qVkHyOH0mVZtguFjR49plDmvDT4DUARunH/LJRDccWGcxDid8m1J/owXeTQ641cJHjgZHrABsLgfA3L1TkbHwStSmRUxA7B9Bg9wOggOxfhJKhli8PYOyL3gJubPX2D79r2pDbZg/nxh+MyKdxi5rtRdg9sYGR23W7c9YNAdImJnYdpbWuyiiz5tSKgA7iDAFOihIngsVlVOkKoIGIksIi4BSGZCwaSsmUrN+M8RMpqEjjk66vKnWBB6+FlUucBJ9HtqJYIk0Qj6DhNFjSd0YP8+65jToc0caJuzoMo0WkxoZOpNJMbk2rE+nOLWlhbda1hp0kDoYiIfS7K0zMYmvVTMQivwm0hzcxltysF94el7JXdGHo854oHwIVwEJx3zQIAjCDeZsxICVlvrKRraqtTgB4c89ROdyCxXRdsvc9Rm0g8eIgUZ3pub6JzbaYcPHxblGdmSpoZ6uQAsgEaI5SpcqjQ1OdCGFZuQGxoZG7ONm+8RgdHXwQmN7a2ttuLq88TH91nvHpNgTQBWlixZbAf27XV+HTBKmoAVhSQ2PPfOtej+E2DlwxfGSj0Hk+PumvDjoHYcCLlITYigquh+nWMp/AN6mmhkMSTIRBQR2AKqpgDQZ9UyVNC5fd74qSJPYvByaDra2/UssjR8pp5G75fM2uDIoAJ0GEu8J8yg8P8K7p56dGuR3Xrw4EEFVbX5Gk89in7jbAahXgzOZUGSXjy5Ovw4bi4qeMh0RXTP08BN6LSOky56kMNO5f3EdFFXicmcHT18RClQfW2dNOr5u/rFxz0VjNSPhyrAKIk0DY2O2LYvPCwlTPl350xaW3OjXXLp5xL0C7fcIV83s2U66SCF1dV5BYq4MaJ8KWwB4mBdamt9DnwaJYaPnanJ039OwJeIIeOjOvW8P/eIi+G1ZAFh2hXYJa4cr+FeuGZ+TvosskearsWfHEYWaWCwX+VpuI3CM1IbN88QYE15PYcSVDFN04TQGV1OakIt82oi5FAJPN+86vNFOmcOHTzo82KYA0NAQ15NLp9oVujEUzBhARSoaMqykxV5oF7R86Apeu/YYa5ekZFPOnrsiCJUvtfb22Mtra1aALIJ/BI3m2d6hUZhT1hn51zrp6M2je12IMSHApHH8/6UZ9ffsMuZp5hCFSMKWvgVKy5W0aeqslqdfDKfAmO85RndOFJMABBNhEIFKxVgSgBIykBYRH4XtxTxgIK0NJYb2RPuq4Q5CIhCQNEbNORXVW+fKEHEXIkvSnD1/f5kuczJFHKnBReVAtlUgJjyMKXS4hk6stfY3KTAT2BRUvEkm2FThJoZ8ZU4AET1BDKB3ukkFoulQobSq64ulWgx2dJwTaO6XfKjwnJV1TJN1My5cTYIX5HqiVLMOPGmJlmI+JnAG7FyauzwYachQcLg88gI2CREvexyfhfaFXPaBSyl5kJYpFu/8ID0dOS7U8Nlc1O9rVp5hbRfVTYuEJn7MILpwqQCJzIJAKnxca9gaQa96vAuPe4pqVfyWHhlJpWVCb93AcV8jc/VQ+SRe4Eyxu91dnbIiioDSkicov3ETYiN5fyGGfkYZQjQvVKgyXNVYSilnd6945E7VoKNxJcXrmpLimOIWJGFsFayPFUuRhl9jZk7brlKvXOc4qVLl9qBAwf0oMLH4X+5ccyc+wrGfo4IPaJCJohUzQZAlFnNQeUC2MWcgCA6AA719/dpNxK88OVRuqNOXKBvnhrr7JxjXV3H3IRly23JkiXCErhZFonNyBefic/dvOUeG5GQkpyH3qupqd7Wrr7SpqbG1aXLPSxatFjz7tiIPgfOu02HBgls/RipxQsRzHRCuTpew73weQ445YTq4fqQceX7lRWeQxPn8Bp8O6cZ9IyDwCbms0WuTPPwuKbgJuo5UuwhSE7TtLQOafCwIOxU4FETaUqT+VMVRBXDnOrFe9U3Nsq18vmaZJ3z554HUcUdPbBzjRQxyLV5QVSywgfVCfmCkzeskRqqX1d72bWxqVFMj4qqKkGRLc0tQvZiDCe4tZdEvcGClIyM4KSlJ9rhQ4dV8QIQUt2aGfSCdGlxctIlG6Cnpzfx5MgGhtEjVhwRp3B0ZMx23v6Q9Q8RiYsCJ1OPysT2bTeL0/fWWwRxXtIFTSTadnSNBgrH1MmDfeNxj6N6+N6gUVBXb6RGkQcPDwwoiub1vA4iJCDT5Dg8QUfHQjc/3AfPhoWJqppQP4KytBmi2zbiBJ4dC8e/OZgKvtM4E0G4QuSmZCUJ5KIoo98vK7P58+cp8GSj5MBfqiqtd2DA0+aHdq1V349gypERW7xkiXYoH8omqKmu1oPioXd0tCvoIjjgZKjzVcN33Q8TQfN9plRwwVTj8OXKy1nQqry+DyCxZ88emWzmx0RDJic5YFz3847wMYMWc8rNNja3lJo3dfNl5bZ9xwN2uKvXyQoSMTQt/FXLL1B2wIZgOLBSoFT544EQvPo0rH4bGhoUYKLMJevSIdFBrJsjJUq8BKGOlRVyFzx8Veum3NVMjsFBdHcZiCDP8Y9TSd7P9fm8cYUTC/dBAdnUlDaUroHa+6zysdLrRF5l4/D5mH5QVoLzUO5g4XHPXJMscHlWaOgodDYi/3u3XVsEg8YUs2vmz5tnBw4c9FNAwMaAPem1wsVjisSw+1EK/0PEBjXin/NQTznlND0g1J727d9X0ogFHQPpqqqu0ebp6u4qQbPQmzw4rJArwG9pU6UCDuYKCyAs3YpWla8tVZ686FBhd979mO0/1OWroxJrRgu//PLzFXfwu+IMjk/IauH7sFyaDZOrUPZARTIfRJM02I+NxP+AM2wIOAccCj3MfLVP1NB0aDKAvHrfNB9+2qN1FW1SSsufvJ50j4yIwJb3xcosXLhQCKiyIyZWzJ0rF8DPgvdIhM+z4ftYBtaM9+HeOHykbaScvBfumc+m7q9CESqflWzwPuvonOPj2+/ccrWoV1wYaBbzVkgdADHYfZwI9a2rQW/Cautq7Pjxbgcp1EAxba3tbfqgBQsWKdh4Y88eFTuOHDooszw27sI7oF7sUuriUaliUZubW3SiOflAsTwAuO64noiS+Tz52dS3xg25WZ60+x940vbsO5gWHuyaIQaNdv26a7QoAEbsekAkHzgMT5CT4DFKvrbaDhw8YFUpwuZ7nDYHZWDo+hcnU6kX7WRj4x58DvQpI8iD4jHQgGKMmlK8hZnTzmcr4E0NmNQ6cA9YPT6H585z4b6BxTnFfAbIHlYp6FZ8NoeR9YELGVQyFj6wF/7OBuN5UW3kT/7NpuU91QcJzsLCk7bh8BU9TkyKY0dAwwvZUUqAKP8Jqhy1uroal+lqblVRprwypwAMTdr9Bw4odyf9Q/bTOZBOoYrgiL9zs9w0sDCvJwBbtHCRHTh8SNaAYKmXacpJDIFNwyaorW9Q1B9AEzoCTz/zPfvliy95mqfGTZMcyoqrL07TrEflQg4c2K8HXFvr0Ce+kWvp7nUixwAQKrl6UgHhZHGSCHjD9NfXU2MYkHii/Pi0y6SjOQdbloVXrp1m6bCQPF/undezCByCUPrgOfzud7+zBQsW6FnPnz9fr6V3QSc1MaJwURS9+OJ1In3W0z3r2YQDaTmBTcIGxh0yZkNw0gX+5HL23ve+1379619bZsu6C4oEZUCP+CwWFFRNAgIELUmNkg/yC3YVB6/aHbXGhkZbcuIJYsP88ze+obo2P+fimhubBLm+/oeXtePnzJ3ndeK2NkXtdXWgdAM68ShO8XB5aCwOzX0e3abOWRWHYOb4BGeEijiNVblK+9mvfmfPfOP7LiuuWINWq1q74pJzlCU49s/UKm8I5YuNRHDpKaW3j+VpkEilUzYAnT/4YQ1CTNOriYNA2PgdlULTtKmY8Z4rc4YyMDCmVmlwKnhFFB9FG5nuoSGdcmIfPjMCOw4SGEfEFqxFYChYTDYk+sNSJEupM5uGU87mYkPx5VIxno3xfKlUCrm7beMVRXWKpKiWF7vSlHetjAwNe5cpxY3UKDk6NqICBf6VEmVXT7ebqrq6ks/B17zx2uu2aNEi6zp8QAtOVK+IHV6czJM3aipTqHH/xRc7GdE/brC+vtF3bOpmxdqoKpZQLJC+3a+/Zffc94SnYEp1WPgaO//zn9am6uvrtWUnL7O+fvrwHH3ErXCyiFmGR3zYMf0vge4pVshmlbLxoFg0ngMPlX+THeCKGuvqU97tDJ3pCWrt1Md94pboWKl3TmlYCqSxKirjJiYQ78l990GBIzDDNaFUUkWxaqbeLiJnoWDHu7ttlIENCbPn+fNe2igJ/Yu/x/eV7ma8Uph59I71iuoxXYJqCVwgJPb3loR5hwaH/lPbNDm8LECuPOXUTvUhuuehMsWZhwKGT7GGUFC4dch0UCiYnrZFixcrTeRm65qa/T114jw7EFN3xDdepEDUrQnIGpo8P+W9D3X12l13f9EFHBLwAfNlw4YV1tfnwBInWxTwXKVONy6GB0KARCmY6BkiZXtHux3Yu89bk2ZF3XFqA6lkk6qZos6DUfRllXINDft9oGeT3Bvv5QIJ7vOVMZGTj4zIDQR0G3FMUNtb2to9xUaGvabG2tpaUg9jTgeJg8nPAbckHZtIGuSZpGz+5RtKI1nT9agY9MW7bxQDh2I+vp03Y4FIT6Sn1tMrvx4dMyw6YAonulDEV8OQpeFwyoZh7wD0JNVHTKxGh4F5T3jk76bc+fhcKEFOV1e3zV20yF5/7TVra2lNPpLFB+BgFq0PG3D2al4na2IqjdwqFm1wrGDbdz7glOM0mQGLtOLai8TKxczjUvbt22fz5813AEO9Zk5oyDGWVFQpD8gIpvCVjkm4v44giWcDs1gyY2lapSt8AvBM6V4HBgZF/Y7TzObGYp104ol28JCPMvMEpCjAiwBOzzxZADbHsmXL7ODhIzLdYPRsVKTZOfEgkDzXqCdESqjq33RBPzv99NPlPl555VWflVeeJlNZRplY5skHNhWZ3X5w337VdwFROPljI/gCKMyubQe9mWIGN8eFUd3iQo8cPqIFBIgJuhTpAj9jgUhH4KHNLlQM0ueeWLv4IoI790e0ZdUpz/Sghn5296XkufhbfBQ3XyEKlgrRNjA0bHfc+VjqX/dCECfkkkv/0UuUkC2ItDUPjyjegy2weqwHWDhVPRYo6GROpXZBBixE4ApE1ELIcj7eFGtB4DU+MaZshw3Ha7B6vI4xqd3Hj5fMNRaD58f7RyoWMK2eX3m5pmxj6mlYIZClfqLIvTwj9PGV3X9Q8ByQeBworFkmETKGhgeEFH70b/5ve+WVPyjOwRKQdqq6+aV7b1JExFA+ThW+Avwa0uNbb71V0nalGAIRAL8DnYoNwEVxkpwckU8ivFm9BynOosULhVcP9PVrE4AVYKIo1/Ilc79okS4KdM3fF1yd0qVTukh9hEgBJKX5N/hsGh85daSU5RU523TLXV7ISHAm17N8+ee1gQjIdJLLoHwPWVNrs9OnoECNg3Hn9XnBrxNil8yyePXFokypQ8KO1g0yb0aTKpzsSNArOLYwYVXM8ZNoErJsY4oTsKq4Ew1KTPIuXFdYPtfZcUAM9yRO/8iwm+k0hgW1UVf28InaYY3405FIpnJ6O/fChfM1WetY93H78Ic/JGyGQ0j8w3VnvnzfzZpJozr05KTKosLAJ6EF9WsRPQqusDmdXjsHBZLPVOHAmzD49wknnKBAqm+AzeCFUzYF74OvB3fHPNU3NmjHHj58SJuFgUR8fmDtRNzk69wQn8vCn3rqyVrY3/3mt7ppzLI49pr5WrCtux71lqfU5oiPX778ApueZpqFyarMaW93WlW6J6BZTljQjtU7l+bJKU1i/HdquCC1YvHJrUVSUarkEjBu9oFq6eLxfJ8TqxSO/rnBQVGnAaWcdeMkFlkVJlkeOpKmZHvAhyHTJkqoJZ/rC+uEjEA0eU3w6LznYcqytLEVCiLWiOGUMd1zjHANelbm649tK2LKtFBJBgSTD/qEmYcASSBDdMzDBDtXVwupwZDj95wW0gsRKnI523dgv33gAx+wg0otZtIJV7V2UQNep+ieIcOkbYqUY+eip+NdIJHiUUNXIwUnPJWBMeH1TU1Ka7bufMS5ZIlszLVecMFnLFdZptFkkkPNuKIXlTjvGBrzGnU265y3JIyAb4+/q+w5ewxZDERQT2G9FpJoHXEjVdVE+vBytNKzEa9A8miF5kFrS6eeXFs+e9QXvKWlKU3HTouMRKoCYub8EARSLPLSclTrWFzAL1Gp4RFMOL2d95Vu0ZQHkVFj8EOTdSIGIAzUIC5q6dIThfkeO9ZtrW2tCqzA6WUVYp5qIuydcMJJtm/vXsGMXr50rRwujJtvbW6Rn2GYMKeEoGg2jEjMgCUQSlbFn34CeWjE54HbRx09KmMsWrQIEfw1NzfZhk33KkZJDWtWna+0Ky+/yArTY3bayafZ7t27dQ3KsS2NRkuEC31+0ujFtQB98llt7e22f98+neQ4XeIMJhPPQgCB4sJefWW38nEYRF4hdE49G5WF4P34s7Ozs4QlsKHkgoRquuVUrj86at3dXcIgnBQCv69OmxP8JBRLmNHHsw7Xi/VlMxIL0a0r2HZkLE3ldqSRz+E6M4/fs0GmvhJcuhzpLm+KBIXjwR/rOip8ndmsPCA8F5RnLrK3p09+n5vid1h4/mRXcZMEJVJpSpuKG+Xhc+EgVSBp+HdV2sYci4cRo9NS7Qxebgy3EOlUwKaoSjj6VWZz5nTY6ut3ajChu+FpKUlcdvH5lqs0Wzhvod4Hl8P/pHf4dnw+zJuu7m49JK7t8KFDRrDLn+oM8qPq6Bh074YGReKwd3SKUtqUKy8T0tjS1KDnxGZQYWaqIFOvAk4isi5e7OVhfs5zBDDzlBCh5xG5ymgSZfGpYbiuDfGFN65geTvnzdV1URmlkMbJ5/V8Vv+gB4gEyzzv/v5eXZMX0fos8/hd16uLmh1K/k6q45Qd998hPBQSH1zsgUOH9YFwvoQNDw9qIXmo3CSRrgMLznFTE0SxqEieDwU7P+2005ReschRueJ3Gpsa9CAYMBiVpYghlPfWeQziIIr3qhFNf/FL37Lu3gGN5NCEiVzOVq+63MYV2HlxRtBdkl/DuolnNz5uy04+WYEsmwMkrSTHopGiruilzCXBrYoLkmvUYWDTV5QLJm2sdx4iETZgEQ9atXTIGslP63SDDPb36Rr4t/x91nsTCaSPH+9RysnP+CKdw18oOG1qVpoLMQX2sFrNAvXLlidhSA9EuTbdV1LRBK+ZN3++Zb5453qNJglcmoALKBUT3N8/oMUMhg5+ROVWsWkdcePGYZLyxckFatzz+htJF29cpr2hsUkLD6QIGkdEzOsw4SwqlTEu3OFFpx+B2Olk5fOCH3kdOW0ENjz8qPVjcVj4o909CmYwr6SUVy+/wIY0r86HJQDv8loRQFP/GVbjlFNOsV/+8pfaLIEQirac0sj4XnDxFBWnDhkwdbFsUutXZwdwdFdpkUOdCnUQUctQDUsR/rGuY7oHClq8jnEr/Ly7p8eWLVuqg6EYJCFydQlt1ABFla3x/04Jw1KiJ3Dg4EEVYYjRgqcYAR0HD26j+PWP3HZdkXIlUXx0XvDQBgcGBXzgD+YBeowSJdYpNaqpd9UMomi1W/X3yULIVShSLZeZyedrZaZggAqwSDNiRsZGZbpY6JNOOslee+01ZQQUQyicvP766+n389ooLHy4iKAzcVNBGmHzPfH179qbbx0QCdPVovK2/LKzrTA2ac0tDTrZCxYutD1vvKGS6FuJ78/G5CF55uINCxFb8D3BrhMTdvKyZfby7t0lBg3Xz7VF0AYjh40xt7ND18/p1eZJaKHLrngJl3QVi7d37z4vswJIqWbP73gAzPOL6hqDk72+79mAtHlF1/LFfdfpp9vLL79sdfUNSuUIltn9vCYsYxwULI827m03XV6UGTSmOfbLj0SPHHktfie6QgFYSLWYncb38IEnnniiHT54wJYuPUk3jAkiAkdJGk1WPmTu/Hm6gFdf+YNuCBkx0g0elDhwSVQAHxQRaNCTeFj8bgR4InqmICjydn722JPP2t69B0XChEgBVezq5edq4Wtq/DMwr4J5wctpDKUMevRoKSJHn0YpHOzXRMNS/AOBIaGSLBTXwCmlhkA0r5gEhJD4ZWjAq4h5ytfHpQg2o28LXa22VE2TC1Cw6ILIuFYWnqZLDpqKZJmM+A5Y2qVLl1lbW7v9fvfLugZa0kBbeR8KbFgv6OgLFsy3ffv26nPASThYUeDRCFa1UG25poheLaeeKD4wXo0T08NCCWtMgYMP55vWCBE1WKZmymmEjxgSkPdZsyBi4qGlliWoSywE9fz6hnpZADB3AidGjfUPDBr1gNjpgfJhbQQBq03awRlAkGh0ZDHxo2WZCvvmd79vv3zxZXHKYdYCb1512XmWLfrkCLmmRElSPSHx491v+8PgRPGemHwCOSzNbJ8vcIh2KLV5eZ4PM1fl5rExzXg7uH+fglI2GP/GXLNp2GQqG6fBSNGHCLuI9q7ow2NDAYodOHjImpuaSvGGqF+ogNBJm2TbyPe5D96bTIwdxqYjHti/392nGFKDrunPa5llK32ie29dUSSvFfm+ucWOHT0s8QB2fwj1xWkTzxwevSpzMzIbUIx54+a2ZlGCqem3i5yRZqAxpntoUGkh/vTAoYMGpRvMnx3Z1wfu7L43SrpRP2YjCeYcn3SZlcRa5XNYiGE06spy9h8vvmTf/+G/C/yAZ1dbU2Vnf+aTlq9w5kyAUUDLasdGIjU1kODmRPzUTLnUHpZ8uNQvEnE0zCaY++EjR5KlchYwGQInv6ba4wi+x/1Qv4+NvGjRQuH/PEOuHatIDYMNzgKxgaLMirVgERU/JJYubOawklw7B4vf4X6Ih/hZBIsE0Pwu38NKidUEIol0HPf44PbVAnCii4P55OTumOkaATW0D3t0yf+cAhC81994w1E3RBCmXU6EDhnBqML3qyxfjVBCmTU1NSp9ES2bnH98rCRH4qVCJk95vRlfxHuRu3reXukl09QCxabDrImGVVll+/fvE3y7+4299vgTT0u8IauFr7ZLzv+MlaXxKVTBcC/CABI/X5Tkujo7dOigTjlwJ1aOzIbXhK4di0MPH0GbyItJ5NDr626psHJsRip8AEsLFiy03/zmRS3k29/+dqV6eu8JRBXrFZSxIKR2xC08B6hgArTGx/VZvAfvSdPo2962xPa8tTfFOs5o4pl4EDolCBpLRPEMXOOll36n5xcnPdwGyqWsRWbbugvVUEEKhQlBQlMPRHnhuI1PTAlp4jXC4EGOxD33Sc+8uQr7CdQJoqAujLZdSYVOKpI8cuSwAsXDR48IyGCnc4qJKagtc8qxKjRa8jvisA8Oq+yI9RBF+m1L7K29e62hrk6Vw9bmNqVik9Nltv1OKnSwSgtWV1NtV1z0Wf6hoBKzPFtiFPOIxUEMghNI8Id5F0rZ1CQSBEN8hQam6pznw4OJPu5ZTrOwWAAABvFJREFUTGDvIHROBfCYJEqgRNtsXII6CkFtczpkesEh+JMvTj6nSzP3VCHEZ494Kq1NjwrYkAYl8jwbG73rlWfMurBxJLyUAB1laalbCYvgKGWSgU+/l9l+/cVFpLkwt21trfIvqnc3NGiXAtzQphMa7ZxoatZAlbBOojLEQ+ADeRBcAOkaqYMHRpzgCQWCwqKtKL5Z+G8CSJBCHoT8N0SDnm6dlob6Rj3gI4eRP81aY1uL3r/ryFH9WZUDSCmz8SmzGzdvV9Mg9KeafM4uu+AzVsyWWbWUpt2PB4YOTCuzy8ad1TDJ94Jq3tFBQ4e7lEhf6d1z7MERShaH9yBd4/5h33JdsSFU+yZAG5sUlgDKScyDBaFphA2BWed5UzvH2vL5xFguFU9KPKxaw/HeHnvnO9+pcSxYXiy1KqkpLS5RvmYri6eFn03OEPSNjxdAAfOSC4S7pTbfKevp7VGKBuEShA5fGcIIAV2qNJoeaHdXl0622q5BqdTsT8BHKbU+FS/qrLe/z04++WQtPr/PotTVNSifR6eGWvKRw4fTA3YtWKLd4eFxa2pDdRN/6Pg7o8zkGianbMfOB2xkytUr3vOed9mH/sf7LFfmvWlsnkgh2XD8OzIIrAlLywOONDFSOR4498TrMZEshuoMtEez4JWV+v67z3iHDg3AixdVvPERq4e76pw7T344MqTFixfJXfG7x4/3yvJkyp2AEvgIm4nMig5dxz8G9WwCKY0iFu3nsjKTE3JP3O873vEOcfkWzsciHJAb4Xq4LjZV5s7NVxX5UHwPPogTTQ15/779DhXWNyilU5ExhgmlZgF2rwgEaUQJf8eEE8k6ScE7cpyPRp8d+Wmda8tHg37C9slJA1o8/YwzlGcTmLS3z9HD7ek5btlsTvPtcQ9DQyPCEQBlvI5g1j80Zt954Yc2p6PFFi5ot5amZsunFqpAwBSApdZh3pdNRZFHRNNUYAnXFVg69+DFEidYsrD4V96Lf3Pdbz91qcz1q6++6n15GhA8LkugBpMCJW+v2EEqpTNYm3loWEr7YskyRSs9D16HYASvI4/n8/k8ov5onuBzvf89uIbetctXXC8CDX64YA6TXeS9d45OGrUhJ1YoJowHQu7HLzQ1tSQz5PNWPJhw3pZy/ELBWaTqb3Mcm9ewu/g5fx8ZGnS2SL5G3ZpUjCIHp3BAIAN4I1p1olmJk1dWJloWppj3amlpSxOovd9eqhaa+Ybahte6OXHeIQOciYS3B5R8EcCSe3tFi8qYVx65F+IINgHXHac+ImbftB4xhzvq7JxnR48csSVvW2y/+MUvbPHCBXpf5upQZqbRI049+Ln4c5U5mzOnU00msHZEBqFRNV+tE8n6+Wn2AktM447NiushnuF68f1oBcxUL735MrKgzg5Suv26bz4jJGe4Rlk6miZZdGrF+DOUKKKYQD66YP5CmXmfHu2Nj/gYL0WaokgCQ1XUph0z5mHGqWEx0cKXJhEQYxrnIXp2InZwgbyO3yO9w6wRaFEDj5vmmubNW6A5LgRAMHz5OYvOaaUbd+68ufbS715S12N9nevToLXHfYHaqfxb6uwdV0ApBm0qnvCQhN+ndIx74Wfcc4g68vv4V1q3+KKoJe5bf58CrUWLF9jvX/q9vfvd77Gf//znej9cBfcWamCSXU2jzvH1WAbFRF1erGlqbhRtvafHadFhBaiJ4PP5fK6ntbU9PfdpweE8R3EUYCtPeqDKCef9sTqk6/xcXUNP3HdzkZSGU8cNR3QI4MIJoFIlKtE0rcXO62bXExEvmDvPiQzlTg6I4gUXyqnhRr1Jo09/Bh4gaDhNV+CU4tvhe+MigpoEygYqxfu4C6AChabulDZM6NFyoufPW2S7//BqqVWrrtaFF+hY5T0nJrwVKXJZpoY5ROqyZgI2YNGWO9jBZ6jXL6lhuTy74+xBjOT3+Z8TxLOb0+6Wq7mlMal4e4eu9/oPG2JEFLJACjHv3Bdw9euvv6YYQPFKuReX2Ozx/vxJ3ULo3OiwGik62zt0kHg9hTUsAxuUplfiJgFrYfKnJ62ttc06OjqV4jmHcdoyO2+6rAhIAbAC3iu0h2pRahkGWXPFZ4CC2pIejqDMcl8U/G5UzXhg7PJgfCiKT6adm1C78+SE0LtIMXpT+dWnS7nsGj8DSJJ4YqI6QzKMmXFhJicnaSHK+/yY9OCERasbZkhB5Eu//40eEE8rfDrXiRuJiN3h6Ua5HDD7mKnnCCSl0y69ln/zu17r9tHoqrZJ+AGk02vkyIuhvBF1dgQLuIbe4z0lxhKHQSVwMZCnbJA6SNKpjYIQh6e52Z/HokULlAIDu/K5R7uO6WBSyeTZxrWRfkd8BTfQp0zOVDsJ+v4/WJZZZ4vk0WIAAAAASUVORK5CYII="/>
+        <xdr:cNvPr id="1032" name="AutoShape 8" descr="data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAH4AAACpCAYAAADtGIkfAAAgAElEQVR4Xoy9B5xkZZU+/NxbuarzdE9ghmECQ85REBQURER0EcOiIobVNbCGxV1Zlb9gWHPcNaC7ZteAeV0TuigrigTJGSaHzqm64q177/d7nvO+1TXjhq+VX/d0V9269z3vSc95znmDeM8v0iBXBPIFdLIV5MpHQl9paN//l6+p6Qn84qYb8fh0C/ONCHESIE6AqN1BHMdot9tI2hHSJMHfvuBsTE9PYcOGQxBkAoRpVt8DAGEYIpfLIo4TRFEbaQoEQaD/0jTVf/yZX9lsBplMFu12S6/zd2l/D9BqNTE0NKT3RFEH/HUripDJZPQzX5MkMVqtNjKZUNfgNYMgRBxFyOfzem8ul0MnjpDV++xT2lEbhXxePydJ0l2ZJOH92bWrCwsYHBxEgtieIYXWIghD7NyxA+vWrdP7/LNpqZEgRYQw5WcFuq+7H92JL/7oN4iRQavdRJQESHkdvp43zXtAqPsIwoz9Lg20hvy8OE3sd0kHnVYdmRR4/TlrsGHzIShmQwSd3T9Lg3wJcaEfmf71CDH8/1vwSGPc9F+/wV1b92GiGqERUeApkjhFq9XSwqdRB5kwwNUveZoWh/cSRTEenmjhqIMKKOQLXaF4IXMhuRm8wCmYTifWElEI2awJXgtoa6DXc9GiKNLfC4WCNh5/1+509Bn+q9PpIAxto/jP4PspeL6Oi1kqlbRBHn74IQwODWHVylW6Lu+hdyPaz3avS0tVlApF/RxmA91Txv2N10y4iXs2DBckoYJELQk+ifgwKTpJipmFRWzdtRdxkMFCE/jDn+7DUjOVUP3GS4MM78Z9PpAm/HsCrh+3kjYcYsSthhTwjecdjPUb16GUzyFo7fx5GlQGkR1ZiQSjyCQVJNSKNEQm5NI0uL1thdMiEPI7F8BWvV6r4ds//TkeH6+hHrURdfiB1LZI/4UIkEljvPXF5yFjSotWs45H907hsINWI05iLTQXmQu2YsUKUDBczGazgUKhqAWnJdDu5mJJw/zC2kW9heDDNptNXWdpaUmay/fZxuB/QCehZYm618tns3p/o9FAuVzWzybkRNeQ5gQBqtUq5mZntaEP3XIo+vv69DfejwkgQODuLUk67r6cNtIGJAnSBJifn9dreW96T5ggE4bI5mzT8TPnFmt4+PHtKA8MYs/EHAJa5CTA7Xc/iKUm7UkHtJeUU5gmiCmrGIhiW0d+ju4rTZC0KcMUf/XkMRx+xCbk+drFvb9Pk2I/qs0YhTiDXHMJmaSJfK6KrKxHKjMVZFPE5RFkBs+QMJfVLcUvf30jbn1sHLO1lsx9p5NIeFqUToww6eDvXnweb1M3045byCY5IJcijrzJ5AImKBaLWlgKkAvDf/dqqjf5XtDalE7j+Z2fy+sMDAxIUDTdFDq3MDfP0lJNz5TPF2SVKGhqJc0rtYXfqfVmIRJtBm+WeV95aovbQP5e+Ll8favdRl5uqI1s1txDQK2UVTBLwbXhpvPmWvcWxLrHMEy10WdmZvD49p1otGNkiyXsGp9F3GohXwTma21Umxk8+NhWtOIYowPDWDM6gHse2wagiKhjG5pOkMrEfyNqydS//IxRHH3sYcjRDV3zgY+klUoFU1NTyKQBchmglC9goD+LF55/LIbzixJ8JsigU8gju/J8hCltdtC1s61OHf/ybzdgz3yMatsEyC9qHn/OJAmuvuxp2Ll3L7Zt3YrNmzfioDVrzBXQLIY0uSZe+vp220wuzTW/+Jo4AIpJqof1LoEbI5PLaYNMTU3KHVTKJUTtSIKnkVpcXESYzWgD+c1CM9hstmTJKHh/v7wHCl4mmsIPAyzMzyPP+wiARqOJUqko7XdbH7EzqYVsQZvOW7Ukjc2sh1kkaYIwzwfMShHA2CPNIU4jPV8my+vxirYpOnGMhx57FAky+nwa93VrViMMUuwen8DCUoRCuSLXOr57CusPGcbCUoIbb3scsbM0iUx+jDjifXTQhyVcevpBOP7YI5Cjdfra93+cTk5OIZvPYXF2Dq1WHZ1mC83aEi668Ew8ZRMvkKATtVBZuw6obAJwsAu2nLTSGD//9S9x1+PjmKjTZ1mA4bUvm6b4+xedi3sffACDAwOYm52RgLm7qZGjoysUsMnP0i8FAbgZzbS7YCbsIBMtIc1YDOKDuXyxoJ/r9Tqq1UWUSyXEHXMfaWwWhM9GQVNb+RkdBXctFPMFZw32DyYtwMogl8mgVltCJpuRsKn9vGfeEy0X/TEFz/9nwxw6nagr+JSCp6Zn6EZChNkYxSjB1h/+AgPnn4MiN5CWzwJDfiaFVqvVkM/lUGs3MTs7q/UqlQoI6Q6RYseOPRgaGcHs4iJ27NiNeq2N4VWjCKI2vvrLe+UAJHSa+JhrEKPTbmEk38alpx2E4449HJk0QfCOD34kzYQZNFtNLRhVr6+QRy7I4PynHI/jBsaRBDk020sY3rQZcaUf2cxJ7qadEQ5Mw7/89e/gvskFNNsddCLz9RRAFhHeetkzcMedt6Ovrw+7duzEMcccI+HXanUJmQLx36npWgi3CWgRGlOPopx+G8mKd7hg0KL+TC4rTeQmu+22P+KUk09BTjEBfawFiabRAcplBmyJgj0KfqBc0bVCxg30i4r/GEMkev4AKVrtlhbcgsUIWZnkEI12w3Q0yaGDBKWcuRMf/EnwykKyCOlKqNWdNh79yBew+nUv12sz2by0ks/HTfOlL/4Lzj77LKxcOYpyJY9cJq+sIuq0XWzEOCdFua+CyalJHLJ2LRYbEXbu2YeJyVk8vGMav3lwL8K4DoQ5cylUgqiDVaU2XnTWRmzZvB6gqX/Lu96tfddxfpVBRtxsYMuG9TjkkEOwAtM47pAYzVaKVUccDpQqCDIbkIYruhE1nODrrSo+8cUfYu98FREFrwAjQSGu400vfibuvudupTrc0f19/RI0NZWawZ0+NjaKYrHkAjgL5LiQXPBcPo9Mu4qwOOjMv5QQoYvwd+zYidnZGQwPDWPzpk363Hq9oVSNLoAmPJfLY/v2bZhfXER/fz+2bNxk6ZpiAKDdifDJb/wSrX33YsXgEAYH+7VBR8dGkQYBRkZG5AYp+HZswhifGUchl8FAedRlCpa5cHEVIHJzcrMkKZoZoDYxhU6mgAwySNKONhQ3CTfiXXfejqOOOlKbJJ/PoL/Sp+C31WxZzBGYBeOO4vfFhSrmag1MTM4pGJycmMSP/vgomkwL40Qug66FmdWmkSxedPZGrD94NeK4jeA1V70t7fo4mp2UMVeMSy65CFOT0+jEAR579HE866zNOOWofgSFQYSVAoLcJgTpMJIgRqCcn0Jq45Zbb8cPb74X1VaLKaQWYTDTxute+EzUmnVF6ktVi7Z37NiBww8/HIWCBWC9QqcGc+GoEbx2LhMqIOPvvannxmCEzvu/7757sbhYVZ59+mmn6TWNVltWI+lESs8ovPvvu0+awLs9+sgjZL658crlCh7cuQ8f/Pb9uPJpwxgaGMTu3bt0X6vXrMGGTRtldnPZnEy/rpsk+PUTX8KmwnOwbk0/skFemRAjfL6v2WigzRRRAVyAb/3bN7B+06FoNprIFYq63pFHHYn60pI28ezsJFaMjiBIEzA2NHdYQLvTRtzpoES3FobIZ/Nah4WFRSzUm3j0iZ2oVhuoN5r4/UO7MbOUIHJ5fNrpIG5GOPfoEZx34joMDw8giSMEL3/jW1Lmf0p5GNgAGKoU8IJLn4PFhTrjEH3Iw48+imIY4ZXPPQKVTBXIZpDk1yE3cjLSJI8gJKDCuH0JH/rcd7BzugFaKKYTo6UAr7rk6Wi2qIFZmTVqH687NzdrQVmlguFh+m8LvJjSTExMaAE3bNigTKJSKTvfYj6RWkCgghbhN7/5DdasWYMjDj9cWsznec+n78RVf30csi7Fmp6dxbZt2+S7+d7jjz3GNkFAN1DGzp3bsXdqHpkkUrBLa8QgkYIfWbFC1oqWwjIASxt/PfV5bK6eg77RMdTm5pANs9rU3EzNVgsbN2xQlL5z507s2bsX+UJZcU2xVEa+kMehhx6K+lJVlmmxOodyOY8iQSKmtKHhE8wQCsUC6JK56bKZrCxBbamBbbv2YGJmEVGUYGZuHg/smsPjuxgQZtGJmR01iTzh5ecfipMPX60MJqHGv/T1f5MqCGDixwgzAM44+TgcfdTh+NOf7kMUmy9dvWY1JidnMTG1B1f+xVEYqt2PTjNC/3FPQWbkFAQMurjL0EBUn8XVn/oZlhqUfILNa4bx/HNP1s3uZ6eVH0vWWkjmt6NjY2g06hgfn8CePXtw+umnC/EbHRntWgYfnevtYYg/3vZH7Nu3D+vXr8eJJ5wgMyNrkBIPyCKJIgnxlj/8QUIblhkfxNFHHWnoYpxICLV6DVMzM6gtLEqo2VxOm4jBICP7NavXoFwpy6r4lOy+Jx7AVP4OtKt1HDN4EVavXG2pXauFdquFSl+ffvaYAnEOC+kYzWcl8Fp1Ud/n52cQZlJUaJ06bX3G4OAACnlmL4w5LPenJSDwMzk9h30T01hqJVhcrGF8cgq3P7wLaVBEGrcw2D+ING6inM/gvFPWY/3YANI4EpoXvPi1b0gVfSaxfEIuCHDB08/C6NAQaswj832YmJzA1MQEVq1cqZ3M6PySsw7HxuqvcfBp5wLZPLKrTgXKa5nEIY2X8MjjM/j4N25Gp5PijKNW45xTjrHgURmmhyzNT/svRvaz83PSKm4ELiDTNAaAK0dHLUVzUK5/D9Gr399yCwYG++X3DtuyRWkU79NchWUY//7vP0EUd1Cv1zDYP4CnPOUpyiYoeCKJDPwWFxcU+XNDcSP4qJt4ALV21SoKNZR18HDw4vwCwlIOeRCCphu2TdeOLYAsl/oUv/B9yjSE5Pn9bz8060tKjaNmA5kcIe+m5FEp5DA6MqwUVprPjZjNal0InO0dn8DiUh3bd41jZmZOIE0rTvDYIw+jkxIW5/qmmJlbxBuveC5WDPUjAP1vB8FLXnsl41kkxMi5C9MYFzz9yRjs68PIyoPw3e//BzZs2IhDN29CjYjS3Bymp/ZhamoGpx67BRcdsYS+0RGkURbZkTUIhtfL58edFn5ww0+wYwY49YQTsfagtUhSQqghgh7s3YMjFBQfqMHswqVhtADUFP5+zSoPmdqiefDE49U/+tEP8OxnPxv5XFYC88ieoYIJvvWtb6HWaMjMjgwN41nPehYKhZwEz6zANhtNo48tLLjsBYxmZmdRKpYk+IWFeW20pVYN/YVBBGmbS4rQSbUZtXXtSrlProvXYXyTybEWYICPNF/+nJrM7AIIMwSRAqFrvH4hl0Olr4yQbq3TkQvqRJHwiUa7hXY7xsTMLDpxCjrq3Xt2Y+v2HXh8zzxajRAnHbcF//mHu3DVZWdhzdgIQOyAgn/xq/86ZSrD3cE8cmSwgjNOPVFARTabx969M7jngYfR11/BYYceqhvs6yvj8ccex/S+Pdi0biVe+pQKiuWKHqCZFtC3+kiAaU4c4QvfugWnn36StJU5pfd/HrmSBXA4O39eqFZdsGXQKYMvoW8Cd3LL5qHnJ+HXjJwd2KN0zL2Wf7vpppvw2GOPKTikmTzuuOOwZcsW9Pf3KY1lbYGL3GzWXexBvD/X3aCG1IUuj7eoPopalm5mrEbA/6TRLjefXZiXxq8YGtFmaneIT1hsYM/sN1WAbIbWKVQAawheiDyBtEIO5WIBhUoRGVqiqI09u3ejVmtYLYM+P8xgYWlJiCQ3RL3Zxt7xSXzz5/diurpEDBdRJ8FVzz0MGzYejBzRUwr+Ra96dUp/YVqS4JgjDsWmQw6SqcvnCgizBfz+1rtRb9RQUjCyCZVyUbs+G7SRaczj2KE9GB4cRJhnKpZFFORRXrEJIQpYbLewb5GbyBbS4NP9v3o1a3xy0upVSYKxsTEtpNA9p+W9xRvTGHst/feTzzijK4ReTb355pu18ShcCpzvocaMrliJhx95GIcddqhuiJAufa3/UnlC92z+la7QinCEf1vaXNS6YqHgAB3TYH72vfc/jF07d+Jp55wrX01s3XCJ5Y3iP4eCp0JRcQw5zCAfpig6wRcrRYT5HJJ2C1sffxyZXEHK4HEAru327dsFz/J384s1XPtPN6Da7iCKAuTTCK89fz0OPWIL8gqeawhe/TdvTGlOozhCmMQ46fijEMcRWq7QsXbtwSoQ0Fc1G3Xcc89d2gAEYsaGB3F05hEUC8BA/wDy5SKCXB5BNod6M8Dw6AYEuT5MN/Nox3l0gixCpEKOzF57HIi733zgdR/5uNIyBmMffc81KBWLLnWCgJCudXDYAS/zuc9dj5e//Ar5P7+JPOwqH9qkSWzJT1NYvHeLzjN44RWvxre+8gUhY9RMvzFlkVTBo3ZyMwQy3VbetZ/9a7278huR36uNJv54+20487TT9Fr/5QtNvJ6hkgmymUSCzGWySv0YzdNjlfM5rXWhUkCmkEentqQUOFfIo9mIUHHPkMmwfgCMj09qA9JFvulD30A7YqU0QSbo4BXnrMfhmw9W4Kilv/B5z025GOvWrlVAcfDa1ejvryh9mp2bRZxE6BCISc2sEKTsL1eUfo0M9ePQ1h0Y6K8oTy6UiwhzRJtyCIoVtNopBobXIghLePvHb8DehTb+8tLn4vgjN5omOcxbwhKgkeA1b/8AOiHTwgD/dPWVCAPnHhJfj/eVQds8fMhf//o/8bznXaJrMrWzwoyle94ieKEIPnUC5ee+7K+vxJev/2cBLMTK9xOig1It9bCSrxe2TwO9Zel1XYK4EeC+B+7HkVu2KENYtnQs1tiuN+g3RiFv0XpWpjsE91kuG0jwMvXlAggQRPUlaXa1XsPw0KiCPX6x8ENwaXpmBq1mW3HYWz78TTRbHcRRG/l8gsvPXodNB6/D8KALkJ/z/EvTgcE+HLppA4rFAlaODQk0YJCkuncUK9qtLi65Wm+iXDKfy2NkcAibc7sxEFRRYP7JSleGwVUWGZZTcwV00gwKfSMIikO4/LrvoFGrIwlYnkww2NePjetW44Lzn4Yth6zDJ6//Mh7dPQ7kCtoI1175SgyVgLjREkKnyJZAKgkU4H1VMbhiGPNzCxjq7/szF+Kj+t4/eEFp6VPgjf/w//Cpj7wfiCPVnVi4sYoagSl7J7+FQQatqOW0ny9nqhjYexwxQ9kRU9ogRKsd4Ikd2+Q2ezV++V6MEEIrUypmtFnzJEi4cnM+E5hlLRaQKxPCjtGq1bFt+3ZkCzlQy5tNuqYsgjCLUqmCMJNDNpfFtq3b8I4PfQHVdgYED1fkU1xw8lqs33AQBomM8tkvu+Kl6dp1q7FuzRoMDvQpcFMli/wOmjWmBQxsmg3ML8wrNWm1Y5nKfBhg3Wg/VlbvRLaYRblS0aLxBmju+RC5Yh+QZJAvD2O82Ye//8x/oBU1EGYI+ph5lwYSnQpyAjYCFm8yKY5auwrFTIJmdQnPe9bTtdkCvjYT4t0f+xz27NmNv7jwAlx0wTnIWu7lavWe1cPCiVUAewUuoVNoCPG17/8HfnrLHei0G8jEEforZRxzxGY8/aln47CN683KxTHe+9FP4pqr3uSw9VAFIC6gIfIGTfOzmOb9/k/34f7Hd+D8M5+EjesZpyxXLL3lYebCzUXLUSnnpGw5MpPCjKGY2UD5e4WxVoUwbQeNpSoeeuRhlPv6FHizFkJLiyCHThRjaHgEYdYRWDJZdBAik3Z0j1a0S5D4MvGr/+av0vUHr8f61atlvivlfJd+ZP7NLsSImNt7sbqoaJVwJMuEQ5UK1jbuRCYXWuUqzzwzQMjiX5hBm/VUokhBHmvWH4of/G4r/uO27dpYbW4qMEJuW82fhZT+QcGwjNL5+7hZQ9xuId9ewrVvfS1ymQI+/vkv4eFd4+4+aWEiHLpuFd706ivQV3CEiwTohFZmpZCotywtKyf2QSECXPPxz2PP1Jxpdmo0MRIzGGN0WE7lrbCQggBf/uS7tUlrrOk7nMCTKch5EXMoCfHCt7xL5eIrX/YSrBstY3Z6BgN9BdUuKIRGo4Xdu8exa/dOvPB5F2KgXEahyHWzjIHxbzEXopjPolzIIlcqIUg6aDWXcN999yNXLiIT5pB1sVcmVxGoVF2qyn1QcbmpGezJUjIY9eCZMznB31z1uvToo47C6NCIBJ/PmW/0VS2PmXMn+jIq38uSIdOf1cEsGrvuwPCKYb2n1N8H1qLDIMekFDFyKBT7URwYQTbH2AG47ut/xI5FFnEIJpgtJZbA6DTPYM5CeTFWmAlk00Rwbzlp4bCDBvGH+7eDdLFcPsccVItJGJiVqDBu4Z1vfT0OWTmCX9z8R9x88+3YO79g1y8W0CYvkFS0NEGGcUsh362tJ6nxANBuyVfyXgnEEOPnfeTiOlqdWEAUOQkK1LKM6Gm1DIXMs9LJIkyWVTWWsyNRusJOAykrZtT0hG4kRSZMcP27r8Lw0ADyBa45sX76+ACFLE19TqhbtmAaPzW5TzB2QjdQLIPgVS5bRCZrha35+TndA91th7uMMQq5BdmsXJLnMcgCXv3Ov01POP4E9A/0qUzpmSI+L2XgoAjZ8ceIGQ8OjSDMpajNTCC751YsTe+WyeEN5ooFpAysuG2zBWRyZWRyJYT5MoqlfoRhFnGYw1VfuAW1CLpBCo4mnOaOJsyDebwHkidZQ0ijlrFhWGpkvuwCIZp9sktYcTKwhiRP4u+GS/B31A5FzTkSOwzdEsMna+VfQruMri11C7nGiNp1wdc0xdyE/EyRJDr2OX4RubAiXDhCYTZfVArMjED3w43SInBl+TtfqwJP3AFD5X++5rUYGBg03oDz8Uzr8rkMSrksysUssvmsyBSsMywsVeWCc7miaFf86L6hYQWM5CNQu8WFSN3n0fX2pNDdNPcfP/Cu9Oijj0bfQAVFLnpgCJonUdCP6I3coSI65rBipB/ZzhxytX2IOouo7duL6clxjK0cQ4YFCNa9aSZzXARWxXISfC5fRqFAn5TBTKeED33vbrFd6Q2I8qt2DeKelrrJF4fmn5NO0y28ESy4g1ms4AMGcYo0dsGW6E0mSNYJjD3kijq5vOruZAGrPiC+Gz8nNMzesWnQiUU8YZbD12nzOOSMfpkBmQiNciEeRXS8O2U+WQQutYxliex++NncuAS2WDEMgwSf+ofXYHhkRByCbM7cFO+3kM9K8KWC/Z4b7oEHHkA7jkX+LJcHuDgqjBl7LUB1adEwEJZkewTfi5P4+w2++rXr01WrV4vlwaqV1ziCFdqhpOrStBGhCjMkD2HjaFu8vGa9jrjdRNysYs9jD2JguB8ZmuACNZ10JQYreaRBCWE2L7+XLw0gn+tDjDZ+c/du/OC+mvBjZlOMSOlDpXUUvMyhOSWaRgrn0IP6sXXfEpKQ6R+lZygYo3wKRCogjXRsU2k8HTWZKYzWtR+M/0ZPyOditcuBWKxokc2ijeBJoEnarfi1Wg0XD9iG7AaOzl0pLuKzhgy+YrRbNbMQ3Ci0KjT9LuAM0wiffsdfYWCgT4hhzmt8wOAui3whlLknqBS12rjznrtQHuzH4OCQTDyYriZAo93R91p9SXEXuX9MSRhBJQ5V7Kad+n2A4Mc/+U5KQCOXz4hkwN3vH0j+nTCj427HaQfFxm5k2nPYsPEQRMSK63VE7Rr2Pf4QKgMVJEEWBW5ZMkizOSAoSvgQm4QBSQkD/YMIM+TlRPjkz7Zh20wTqk7QVwZMVag1zu+H1CQgK9Od4NzjNuC3D+xyTGBHLdZdG3tIbF2nkWTL2LMAMS1DYAJmakaBRdwkjCXSZZKmuAmuTE36uEyzYyZRGXRtugrHCtbN9RSaqIXc+Lwjlpup8ZaimZknN5/aLvgaMT76lpeif8BKtdzkSlkp+FwW+XwokkcumxEWQB4e01fB3glzfqDFmCXOY3qpij2zc5iYmRNPj7WCyZlFTE3PaN2EzjLnT0l3zyC48Vc/Tum3izkLSLxv5wsZFPDqeQoOQH3mUQwkS4iSNhb2PobDjzsJcZpFVF/Avom9QGkE+8IxzHcsKm52OjK7LIIwJ+bNczGYEkqzyRlfrKoQwyCKpVLyyK3yFWL16tWCbVetWiWK0Y7tE2i3UmTDMgiRkGxA16SFdSVaU2fXTOCid5pDWS9uD2/JaBIpdPpD+VwK1Qo6PjXzDFlqqzYV1yS0ErIIoO493WvyNY73T+toG8SII8IFGE+0m+b34wh92Rj/+IbLMDRQUVWQ68/r5sIApTwFTnOfU7DXaNZw74MPYcXQCmT7BjDZifGr/7odv/j5r7CwuKh7bjZaiq083Zv3q/RQjSP2DFIoupxb/vDrlB9AOpQ3W3yDSrREk/IFFLIhGgsz6M83sDQzjrSzhKWp3WB4Mrn6RDyydwaTM7NYmJ4WLNpqkDHCsqpl1wGjJUdOZIzAxgOqCYMaMlomJicRODIGF4qfS0TO4EvL9WnGy+VB9I0MYGx0NTYefgRWrdmARx7eiUZEDJ3mXi0SXcFzc7HkaigZwRZWDU1oKrSoGhd3N4AyBLo2x67hhvELpss6gEaBo29scBU2a6rgpjMLqTuReTerwcIIf8fYQTy4pIOV/UW84xUXm+ALRgRlbJPNBMrj89kcClTGDNCoV/HYvgmMHH0qrv+3b+Kmn/wUzaUakpibqS16FtNgGnLdpweedE1bG/8l2Pu2229OuSuIEgmWJFWnY61D9LnFfBHtZhXlPJDEVTSJ4i1MYms8jDu27sbM9CTI0m3WG8rzSXpQaZJa6FKIgCkSF5sgBzlkDeuCUTqmbhLyAai9xgX3xAziBTSBSptUuOH9RdIkslsYMwyvXIGD1q3H0aeciU6SwfT0IoKYKZsBJGCwaF5N2YMv+lBI0liCMNRALprzvd02JII0PW1cerFr6uBr+JV4eM9bFwnb/KhF/wbskC9HgXdY/ubnJh0cubYff/OXF6GvUjIGsKvO0UUJwMmhtTQAACAASURBVMnS7zM/A+qDa/GjO+/Ad7/4RSxOT6M6tyRhE71jzKB7UZxhULDhLz2Bp3sOX/0L/njbzSkrcTmmR2J0UvAdVYoYZbcaTRy0ZhSt9hLSxhyqrQQ/fGQntj7+BHbu2KViDh8iH2bRYTWo1VavF4kN9CX+i5pLIERmNKILMHap98Eyxu5GuVA+q+DfvQYyWOli4u5B+HTtVhv5QgnDB43h8GOPw4bNR2PX3mmkCWlGXATD9wn3d3NZ19JkqRU1uCPfq9cR/OFiOizBP4OYSq5nwN+HzwR8XYBK7zeUrbxzEdlQkCvXlqkc1+ysI1fiZRefp3o7LS7jWaGdxEyyxO/p5/OYHjgIn//eDbjlxz9WQN1qNlBfaqJea1hmwazF1ROM9r1MF19Wc2cRfX3k97felAouDPkhbDeyBgfGZwsLCzh43TraAbSjOqr1Or53z0N47MGHsG96EvW5qpkR+lpqRxoKsFhYnFckOjRozYsKimxFtC1ljrgBGEGLlNhCqVDosm60GZyvtZ1sixfzvU6jFMn3PCT3GO89E2aRKRVxzMkn4fjTnopHH92joE60aaVUbocpTTOzTpaQNmTbCBPmmy1OULDnzCbvn7IkV4GsIAV+jlhpG8HKjbpfFzjK1MsCpOqGMaoXsYEEr3j2GTjz6E2oVAhG5RWRM0dnUpvPBsrfp4fX4Gs//BF+8Z1v63lb1RqYWSxVG0g6ZlloKUzY5t+9lRKwxKyFn66mFXNxMvW33/m7VACNfEtGwdxAqYJGbQnDI/2Wr6YdAS3fvO123HHbXZidmUCtWrWOGknGkSmcxs7PzWgB+ojiuQVQlbOnGdIvKv9OCJMwr1AnSlDWzW7UUDHv5ykkBkl6TMtZXb+sqMxOQ/3DFQf7cNqZT8bw6i0Yn6wJE0ji5cWhn+X1fDCXOFPPq1PjPa/fkD7g4tMOw3Aphxt++wCa7Eejm0jNaoWsx9HfuoYNWgLhDS4IzKYBWu2aijtJRFcX4W1XXIzD1q1EX39ZcY1RpcgoNnpVe916fOM3v8F3P/tZ1BaqhgoyaK7VQeNET8brdxtCVX1ZFrA2rCd8sMdOWY6hecG2HQ+nytPNXuDxJ57A0YcfoXowIUxT1A4e2LMLN/z2Fuza+oTo0Z1WJLSNC5QLrSDDYExtU0xX2EjhCjVSBEGvy3mPj4yJhjEIpPb5WrUE3omF5JnGEZQx7bTXE41yLdRsfHAVLW/GTUUNDczm81ixcgVOOvNszNbLruHTbyrfsGnBIz/TbzSfx1twB1TyKT74mmcp335g6y58/IbfWZSeWPA0UExx9tGbMTg0ALJvdkzXcPeje9FJXJFILeANtJsNVQJzYYLrXvd8rBoZRH9f2bh0LgilArI28rXHHsO3P3s9gnobs9UF631okyzJFJNt07auXmFo0cTjd7QuAW8eCEnNTbJ2IcewbeuDMn584F27t+PILWSjLGtbSsJDp4Mv/e5W3PmnP2FpsYrFuVlpL1E9+TYX6PhArN1q6Ca5YqwZq0ecrcmwuEFsWxclCxGLY3HLuNhWwrTAiF/LdW+XirkHUBqnaot1wfhWKh9t+9hAGiQwpIC1h23E5iPOxkw1Ul4fKge21IqWjXi/zGVkm4zBqQI0JHjds0/BiUdsEMBF3ttbPvNTcQUOO2gIVz7/PAz0FY1k4hDHWr2O93zlF3hk15Q2ra4dR4rASW8uFXO47lUXqWuGtHFDLRkQk4oVYm5sNf7hfe/B1ONPoF5toLG4hEg0MWtKZdm6G++4YpoXfJeswt/njJwiM2+9WsaDePSRe9K5+XmsX7MGCCx/FnTioMqApcMgwAd+8GPsfvwJzM3MoN2oi03q4dzeHnANFiCCRi3nYjKQ4W5nBymBA0er9bvS/5uoIXljZMowyzDs3ARP7fZt5f6BfdVQ+DbNGbn0Dnvw1/RWhdaHPpQo0Nia1TjhjAswOWtAjG16mnWn9Ywj4tRtVFcoCgNc9+Iz0NdP1GxYz/APn/gOLnv2Kdi4akiVSNKoSZfig6saFkW48iNfxu6ZljYPg150Wog7LP7EKJWL+H8vvxCrVq2Uj1ddnSRMRuO5DH40OYWvffjDyKUhlhZrmJ+ZU3Acta0TNqZ/d5aOz6D18B7Qde/qn+x/cJCzBG/BAIId2+53Pt7Ff0w7HFNUQUkSoBp38I7PfwFRvan8ul23smTiWpx1QZcoehCIQmfpVakSc2kGLs6HEV4VE0abzOWdaqNqSPs8iMRqYLPe7sKdPupXHaDXnCk1dJvK5azd6N3FCXzkTDY0GHRwAOdc9Jd4YjvhYm4qq6AJ+KHQ9R/dHwXPew9w7UvPRH9lQIUUami7k8itsXTKz+qrlJV6Gb0a4iy88rp/xXStZe1EHSvwsGWZ3/vKeVz3hhdibGRIVVG5L7c+gysPwT/dehN+8JnP6P6qMwtoLbHjJ2PDHshWcmml4hkH0BizyBWaHALLTKZbZHOMJHEHd+14kFVHV6PmbjI/4YVPwd83PYWPff5fZY7n5+ZkchTYREZGoKaxYCKBqJKX0YL5luGUwxKSjh7MdhzfZ2M7WEnTZ6n6xc+3yNkHcHFkkasEaVmquXBXePGbRDEhNcBPvnCsV6/9phXcIHI4GFq1CqefdwG2b20gn83gnGMPkRn/7n/dxZKhLayvwgXAu192FsrFigRPIVHgCgLZxMh6OmOOuC0XwveOT8/gTf/8E3EXhAa2WNjpICVyl3YwUAxx7etfqALNgOfOuecc2nQMPvbv38RP/vXLlAZm9hHgksd1LsjRz3rmAsiUZ4ysaWtlcDV9vA98icR2K5+7dz6QygcIraLf7MV4yBMP8YddO3D9176h/LK2uIimIw9GrUj1cC6l0DUKm4tSKNrCEaZkBCn/Sf5XR68hN73XHHOz1KqkdrnUR8iYE7KCq9AKHMs7Qu/3voubVQ/sQRS3v2je/UQMml5x113vO987vGoYz3nui5GPs3jSYSsxumIIP7nlQfz89ifkl3NphNEVfQg6EV777FPEFciRaCJuQkEAlPAOdSDF6sSp1uoWOacpds/U8Jnv/Qbjc0TW2GjSRqfFGT8RBgvAu15Hwa/A0EC/TcfgtqcVXHsoXnf1mzG5fatKzlN7JtHh3IGOwcm+zNoVLhXJTwhxZFDx7DXQwp7ZK7JiCf6egtcOcRUkXwZ1ayfB/+qhB/HV730fGbJLG03l96VyWRE/YUMPanAgAS9M02XRsHWMdtqRmjFs8gQrgMbn4xdNF+MC+kDW232TJFXarsF766mC9RAlfflYZt5tPrZNd+MIEhBcOsWF55qqGOKsAu3Ohk3r8fn3XgeNYBChsw0aeQFMCjzbyDgcgDV1wxCdFWIwB7aBM8hNMTXJoQVVDV/Khnm0GzU8MVnFxFwTESNql3qxBFUuhDjs4DH10omHILIlkC2vwOLAClzygov07/pCFZ1mB20Ol2p7opdLZl1G42XmgzplG07wHAph7CbPHbQAO9i9/T4J3hcTlArqhYa6Maj/z4fux5e/+31ZBX6xyCL+eQx1frL/2uBJE1CxaItLTp5cAtOwTgdlNxjIm+dljSWJoGpUoR6Dw3TQz74hgdP8mQV9rO759mb/wIpJnCWggBmWW3rJoIj0Lr4vRSFfthjFggYce8KR+Ke3/r3VFBw6YN9tuJBCHocRMCAkoqaRCMp1m/pMVtHsy+BpFmvkXlzM0VvA6xZKHIrm75vSKY1swV21GVz5ssvlPmenpsCCe6tJi2kVSJE/3CaSiXdarfV0d2FO2PrzFN84S2DE0RDBrm33plbNMTOrFwtbtxunlm+dmsK7r79eo7zYfz49Pa0LksMWkbNOPyZcm5W1SIKXRlOQbvAAr1UgEcL5TW9R+JnUdGo+f2Z0T7fAtmUjL/ohRRYjdWnTLK0q1bL7VZroNibzYFW6OP6M07ESG8ZEU88qPI2z0kg+tWvHPvPME/G+173WWQubKME14OcRMeyicc6dMDKXSVfjlJl2GzbkNjvDFlcA8trWGzQ7jnVXG7VJMgWs2nQyfrvrYVzzt29WlD89OUX+F9qiSpu785u7m7Y5KrndiOvqcZiAXusKNZIZ14qbYPsTfzJT74TufYU3lwRdluIYV33sY9izaw9WjKyQORNAE2bEvo3qNk7MI2Z5ES4ziv797zTPxhcvyHdj2ZIkxowVaRrNpjB3sk206TizjTmcQ798dcsTNdQz59I3+XE/G8fh1EqpOJPGaYcWSUkE0zZHRhC1i6VMoNzfhysuex4uOpkNJS6ecOsiDXVAUrfjV1mLzQEy6Hg59LTgys3qcTvcv6Z7bTapOqSQm0XBbHkEJ552IX744O342LXv0maan5xGu2Fz+biBvUWWn3cWdVmbrTZgf7PmjO5XYAJn3CNTv/WxO/aL5gwNNRaMNgHBlzCDN33ww9ixcyf6Kn1inwqQcflqa8nmyfmgg2wer/FKP8IQfUxZAvpO02JW/riYziIKtrWCg2kaF0OQqcMCLE0xbdKmFI3bNpt2tcP0lwNEe61gaPc3EiK50RgzeOugZgfahlwGI6uGcd0rL8eqsgE3VoFzNWz304EIoyeKShP3Z2Toc+lQ7AeLDZQ1+c3gt0vQUUo2sPpobDzyqfjmrb/CZz/0QY1dmZ+YRrvZURWOFsBruy7hNJ2/M/KKZWTmEi2GkrZrjay+z79L45949Pb9BO/RnS7+y3AmCXHVJz+FHTt2mUA5k6bRQKlYUdNhxFzbTYOU5udC5IJQ06fYj81FZMrDpkBGwuz0ILmQr1XFS926ie1q23eiIkuPxKaxFE/+TNQsg2xlrknRJj6uoYVu0uMBdCNR8Xt64nxFjUGnf5+lPMARJxyGa156ETLUSEfA6DXRvaQLm79nFT1vgnutp35nXG5Xo3d7wAWtXY/sovK1R12MFasPwse/+Gn88IeMqYD5ySkkkbVs+U3vYyMGsvwitd1vCG/apRgug/EKwPsVY5iA138neAV33RZhUpECXPu5f8EjW7dK4H0D/TKRHkWrL9ZMu5wPCYwnpfStVMx3aT/lkk2x5AJzwyzn2AGWFmwciEG1ROIsImcngP8d8XTjsftq1HKRpGsJnDb5a+vhGR73jEZl4YJfrTpHlbQVRKnuEDeRLZbxgueci+c96ThZGwWBPdMovUXxwv4/v7Ms263ULTd2UOhe8N4qHHfmy9AulvDcv3yumjKrC1UsTs+ps9lrhH8uWVjH2OFoWD+mrbsONPU9FrHL//f4x4GC38+H6Kksgvz6D3+AX91+J/ZNTmPlihER9Kkt1NzZqTkJQ0T+lEOEbKJUg+PHOEdOXaaWRlhbVluRsebcudIqW6v4ZRUxC9i8pgkAcUQNPxOPVoAFE2M1G2BB089Ie7nO76ZfMo5wjFsjaFre6ytwvjpHAbA0zf759771FRjmbDqW5vTN3tNl3hxQl/ea7u/Zm3OBNu4f9gzuOiqp0nbbv/m8p5zzKuyLY1x8yYVI2x3DTJbaypq8Jve6VFpemfWsZVPe11NxVJ4mXOuCX+HzPRhG8PgjtxnE63DcA4M7H93f/8QT+MfPfRb7xqeENDHlZb5OwU5PzMgf2pgOju0IdeP0nTRRjNR9p6lpl6dsW+uxiBcy81bb94vnYwbTKm/q2aded6NOjTxiqZkPZJbnxskMujSG16LwhEp2HL5AUEn4dyR3w0IKcfNGp4VDDzsc1778Ik0IEYfAWQxtHIcNeJN7oHk3VpFx7Lw2+2zGx1tiHYnla7uCKdZJT389djTn8ILnPxedelvZUmOxDgJlPiXrjb+84PkZJlRvqYmeWvpLOSnO6Y5pdXHC/yR4v2M9hZQ6e8Xbr8bknnGR+VeMjarkyKDFplVbfkkiBunCNKNcNM1+4ZQot9i8GU8j5mf48aX8O6vaxBMOFLwewOHntPISpjRcW9YshWRqpeVljTfT6tunVWdz2YgXGrEDVhKXLUyKKG4jzGVw8bPOxAufdCJsAJ4Fe70MnD8TuIJIY+76Qpeyu57ah4tcZOks4+GfmXEkOOWcV2M8buOSSy9Wl+zE7n2qzJHZpC9qdU8rOF2WBW6ub8CGDysG8jELKdi9BTFqvnoi/2/Buy2QBnjde9+L6YlJ1BttteV2Qkb35JSRTsVBBqOYn19AqZRHu97UBAcxWVUAsRiAi0Vs3LTBEEMztQQnyJV3wEi3b8+CPbJNJHAVAARDIAxp1m3OjUYnyGotR/8+4PK+jhrPh+a24ZeqZq6+73237iVuS9Yjq0bxrle+EKP9JBwaC8i7pgNNe9ctuUaGLqPVW9NurOAYPb0ECsZHYQnHn3s5HlgYx2svv1xDlnZyXm2DzRd+MzlAxltnx67pFmnYs+i4CrbZrWdgOZay6p/WsVfwvQHRssZ7wQPXXP85PPjQw4hbxqAt9pUM3NCM+hhjK1eiVquqVZjATnNpSa1V9SUifSZ07ThXRyf6Z40PXviU3XIwxfuhpis3pbhcNUlpXcrJkHy9VarYR+bUwpENliNtmVJqhhtQLCF6mJobxY0oMbCIrNsYaSZALk1wxMlH4e2XPBMJ81ovfJ/f76fJPtbowQDE0LGClFHUjPcvSmRP+sshxtlwJU4454XYWp3Ei1/0fAl+z9YdaNVZOXRkDnLundnWWtBqGBnfSCeCqx3IJUw+g5C9DS7rkOvz6R0F37sjvL/v9a/ezPzyjtvxuS9/w7LTJEFf/6BAEuaM1Wodo2yhyqZi3HYaTTSX6IsLaDc5A4+948s0oS7o4Lhv9PMH+kx7Tw/BkprB4TBuSoVnk0p7e3y8sUwcO8VtBy2My2098GHgi6F/QtkI7XYJl4mme3AcyWUXnY3zTtwiq+ILJb1BXG+6p2v2cvV6wDF/T5aWmpn3eX2mshknPekCPLQ4gZc+7xIRR/bt2IW0nWoEqwJAFyAIqnYceW0gujONRjGkUabd+3xNyzAOo0y8h+T/O8FrZ/QM9vc3vGtiGld/7GNokM+dJOgfHNIN5Esl1JaaSvM42WpmchqDlT40qkuW57rOFAqeXz618IQLQp0+mjeTq080Abvac7cq5SY+9lokWROhaMZt90CP37wezu1uZpfOMeL2kbpZF2sX0+9oxrKhZr2vPmQjPvjaS01QnAbta/zO5HqLpXtydGsfzPXGAQdaUWsGseccXXcqNh5+Kn6382G84YorpNn7du1G2OHQZXYYWVTuhejxerOgoWb6UuNVYXCC1wAoR34xsGx5uNKf5fFeyH8meAVQKV7+9negsdRUF2uhVHInOXCEZoyBgSHBrgnZpBwQmMliaX5hGRNwJUW2QcvvyiVTUNY9Y4vEvWScd+1mZ+L9QtJskg7uLbsXJr/3gjzK9Z2Aeydg9UKdGhQgrGB5uD81nuwWfn6x5Kp7UQcnnnQs3vr8pyFhAEuouMubN+vXjd499O2kvHzfznKpIdQFgT7RC2Ks3fxUrDvkWPzbHf+J9//91UJMJ/ZMIMP5/4504S1ibwbmTbfGonhwxroQDFdx5p9TM2RlnaX5M8F7s3Wg4FVxSoFXvfNd6h1nixRBbqZz9DPs1SItScWWZlssXVbXmrVal51DhZF2OJ/LefDC792pE/74Ea6Zh0u94HtNqyyGI17sf2iApYP+iw0XfA4fsXdNsouC2XBh4IqnYBlvgMEqNy3rBmq7Zg09l8ObLr8Epx++1t7j8IflWMG1TrvY04J5l8FrQ7syc7cBw0f+/FuMw4+/GANjB+Mbt9yIT77rOmVDCzML6gTWejm+nA9Yl92FabH66RwobHgJXSLHprtBEY65a4qSLAd3+5khsTmWmyGW/5bic1//Fm659143FaMtrlkmzxw5oxnsNJXkp7MnnKldwBMZ2k2n4baQojVp5y0f9GP9ZHxI16Xrkbb/5lAkE6blrUyXvNb3+lrNv3flym6q5iZlmbl0ubnKrsuRtoKv0NURHKDE/J7CXrlyJT781iuQURVwmW/vJ2n6dTrQvNt9LWMBFoAsX4P0miNPuRylgWF89LtfxLev/4Lq8NXZqsUVztR3i1yyGm5su+M19Lo1tZ7J3xPSJtBlkT3nBHD+kCJ+H9X3Ct7vpt6gjxuVulptpXjLe9+thgIb/l9ANh9qxh13HevgnAUbtRqqH7Ma3G6Qg+5GjKo/3Z3M4HYhP88iV5q1XuybUzCXaWD+HjXT1VGfeMxIt1DjxqHZ/RsB06dy0pSeYr9lGGZ+fQrpFZQuzUWH1nDBOCWw4connHo8rnnxhSb2nqi+F9b97/L7XsFrI/QIngcRHfekVyLfN4D3f+Oz+P6XvoL6YhW1+bqUwbtf8fnUEk7XbVmO/8+ex9rSLO21vn/OxPGvMSjc4RqPPfzH/blWzkQtw3+2BqoMyc8neOW170Lc7KDW4I0lqPT1axIGT4KgeV+YnUfSbttkKJ2SEGkBPZZPky7SBf/ncHdNvhaH3wSvmXZuSrSgzq4sXErYZdosQ578DAIcytVpDTgqNJsTx603S/Edtt2mDBdc+nEhSiFdKZYLau3ONpuWNunNf/UiPO24TeikjAF8N+z+Gu03wn4Rv13VxTLELXyXTQfHnv1aZEtFvPOTH8BPv3ODMqOleTaX2nxc+3IVU5uNLlqV/u4yCV+UUXOGS/2ISfrfi1vAYhrP1fnfBN/VMHd+mvdb//CJT2DP1JR8PRejUCxr5CajevLp9uzcI+5Kq9HQOTcqtDgN87uXBRdj4jpSINMxtmARPOkhG0gj3YSpZY1f5ot30yEH3XrBy5wTruQGcaNWbJHoIhxh07mTLnjj0tRumCDNdBOtuufoNTE4Oop/uuYNqGTMTRyYvvln7NX85Y3gy7Q9pj6NcNLT/kYW6lNf+wL+5bOfQaNWQ7tu8/a94AlWeRTS8jKL6Ak7+9TWc+q8sBOljL5knopnL9i8V/B+d/aakO5iO43nv+fabbzlPe/TpEvWszmtqTzQJ23rHxjA3p27kXYiDdRv1xvIaEdyopnV5mlNBJa4yF34ucCpZbMuLXcVbvu558uf+uBOiuLDWqmV48eJ6pjfZ27PQoUGASjiNW2zcwNcW3NPV6tcjidhmC7p9dZfZ1VCC/5iHH/8Ubju5RcjzbigqtsHv0xqOdDk27+XBU/6uTZJ3MbJ578RnUwGV13zd7j5t7/B4gzZzHbGzeWXno+DRytYu3Ytthx+sjSf+AnHovArk7cDDLiOkZo3OqJ38/iS6mIVu3btxPjUtNZgdMWIxrsHjz5065+ZehmVnsHCvaaeP9Mkv+Kad0h41PhOJ0D/8KBQqpGRFRjfvU+CZ3GmVeOZZ4ZW+QYGCp5+U8CJS1XsnDTDnHvNI9l/vRG9F7/OaaPA09jGnrkqneBLsW6tVu+jenseG0fSi5z5wMtyca/BDvVzgRWbQvjF2IQ+ts5zdAb68YaXXIInH7vR4fcuqncuwt9nr8n/7wTvLdqJ571eJK7LX/ty7N69ExM7d+tcnA/+w1+jsTSuruX+8iBOOvlctOheOA3bATtqi3R1CmIZhgoukzbM+jlfryyXnTQHCt5H0YEt3oEab4fsxPi7D38M+2bm1KPNHJzjVGTys1nMzM6onMlyIjWe5XCBIq4Y4mqpsgJ21lsGhaLNZ9UZKgfUwL22q+/cgSbGqzNwg0ebLAekPZOhHWDRfWgXqBhGYOe8+SKP105P+jBugINhXVRurdNWziV5k6dPXn/t6zRShfN57b7deXvupn1N35t/g2z5xSPI3FSNNMAZF1yJJhJc8BcXolpbxPzEFJ739NNw7ilHKzvZu3cv2u0ETzvvL2y0W4YFsZY1RSqEtuYILU8P/iHShYO4FfASgeD3/03w+2m94FPpu4KSG/90L7763e+KK+fPNB0cGsYS83Z+eMeIGA1W55x5p6n3QZa5E+ukocayuyTmQAP23HVbq5fNpu+y8ILndcjtY0DpgzSZbwEX1o/HyFb5rzv7zaXConJzg7ISyE3D9/cya/wm8FG+ByIMjLHNEDV5wEEbp55wNN7xmud13ZQ/dsz34nvBd69Jp6TYhtVIA384NvbsZ70ZDXRw3nOfqfR3bnwSV73kAjVu0Idzrs2WLUfisCNONndDy8Jj3kQbk7S1bgKyZLKZvtHF+U3hu3pdJuAF3+vfe4M6X8mSeXQRqRinaYqXvfOdVp1rW55bKQ8Y9ZcTSjkgoVnXMIBC1qL9ZsOgXp9XMxU08gT71SC3wQKy9c7v3z3bTWV08C6DthBhjhg1I1gKuqPhTdQ4agg/Y+P6Q/T7J3bv0nc+QYFM4E4kgKRUKVvzB+/XUbcs6nbDC103Tm8qJmBJPspGnw8OD+Dav30lDls5pJGsjPIP9O0y94Ejk9AySPDGG6DP56HHZz3z9SCP6annPRWduIVocQEvOf9EFDJZNHiKRpzg0r94EZJMCXc99ATufPBe3PfEds0XaqlBdRlml3vTBDHWsK313GIcp/H8+ZEH/7AfEaPrTx2I0xW88416KLczrv70P2Pv7nHU1QiRiK9e4kmPBGg4cG9xHs1qTa1XFHK9VlVaVGBHiqNQ+SmWjI2I+ok73jMU2PPIfV+ZzFo2QKWYRV9fCUdsWounPOVMnHXqUZpLx5YvBWX8X8+YEl7zZzffieu//WNN6uJCsAlSvt2Z5WV83R5wWfPN9xuubwJM3TGqTBU3btmCj7z5cimdhhj3VO+6m8ALvksv94pEjU9x1oWvx2IS4YKLL8D87BQKnQinbFyFUilEK83h4aklVJsctJxBJ43sEAWlecQ+HATuXZvj01tKu4xzCDQLHHT7yAMH5PE96JaChG7o5wbEdcsnwHd++TP85Le/F1onDh1CTa6iH6HpnJ2e0lwZGh+mEJx/y9/zNTTBbe1U46bSzDdaNVWjSOvK02wHGR1Pyu5RNimefczBuOaNL0auWEa22G8bZL9wX2Fo128vM1qXq3V8psvecDWaHfo6etrlnOrLdQAAIABJREFUUyVoxs0aeaH7s++6oY6GBSt9SvxxqHRRCS574bPwgrNP0LHf+wvebWSX71NYxuJxfYc8H69TwbnPfAlum9qFv3rBJToAapAzfJMY2VUrdVgz14vsZimmKw9zvT1NWemby90Va4Dzh/O2Pjxjhz/buA7boA/ff+v+ZdmeAwB6BW94ke0C3TiAxyfGcd2nPt2tvtHskHdXLvcp6FuqLii4o49XvskTpjsWCFr0buNLKBa6DPo6FWs6ETauGcKpRx+FVZkW+ioZTcV68gXnoNTXr5mwYaGvSy1aFsufC94s2DK/3FLDBB/90vdxy+13q7ikESqOmOhNvQWLPqOwdNQqeNZBq0O1dW073rRvbAj/es2bNQv4QMHrda4L2QteZVKXiTQ6/XjqBZdhW20ef/mi56BVb2LLyjE8OrFP1TVyA3RapROumLLi6RlY1T1hROtMZI4HkCyPPekOqGQzhevuleC1XC5a9qdGdjnc3VV1gu+ZlUYm2LWf/5waLSi4Rt3OSunvH5QF0OTLZktNlS7YVGBF/63+OlKtoibWjo1gKBfgyU86Fcds2YSoVdcD7dqxC7XxvTa8MJvBEccfiU2bNyIln8zNxe2mTeLjOwxeW9ohjTpE0U2B8IvvovrPff9G/Ow3v9dG8C7OZgAZ1cprfm/MY0pj7dR+8BCZxwxKTzzpaFz7+svUb2iwrxVgzD0ai4auwCqCdm6u4vvsKpz5lOdgMm7iac94Cvt8sFSr2rkBpYIILzygkCCZGkRczq5Yh/UIxT3ugV3NPpfJWYDrqWou9uJhN9qu/5PgvU9d1qYe8KHH/33qhhtw59332KSodltBUqWfB+GWMD0xhYQDfHnkB4mYmVCb45gth+JVL70Mmw9ejdt+eyNKGaAl2lVq57W1Wf1b0oOPrBhFpZDF/Ow8CuUsTjnhKE3PDDlwWX2qjnPnTpdga7NFuAFml+rYPTGDJ3btwa6du/H4jr1a/MgJNYMQe+d4+JHx69XoofEtHk9YVohebIGLHDUtoGUBhCAWZVmq5PHuv/1rbDhoTFC1xQn+9Gsz+ewgVgbhLAp/Vxk7AkcfdxYerc7geZdchAyVqNUSNsIDhIsDA8gXy1izdr1AnJGVI1ixYrR7uBKHJmkABYmjUUcnWEQ80pTdSY4E09DcnQABEUhO5/CC7+5q59QP6JZ2Zn65YGBPFePGu+7B17//fXWnkBUqfD6bU8co/dLsvgkcdtBKXPv2v0eZGscFcQ2PRPTuuPVmhARIskTAlufMeoKCtKbTckeXt3Dc8UcjIjBT6dO8WBFn2XHSbOBHN96E2+5/RFOz5xc4vIEjWW0fdNpskDDNZuuxPUkWHNPKgMdAneWDE4Q0us1ghxQ57pqbasXOVf7dmK02pqUV1TE0PICvvu9q66qVK3DBoOPiJW76tbFmLfXadPRTMbZ6C+6c3o1XvPRFiBZr0vCxdWtw/AnH45o3vQOtbAGLSRNtXoeHKDLOIOdQQE5TgheLiC4kxz5CK+ho1Bt7DgXKaWqwgu//UfDLhYHl+vay1V8G++ZadXz4X76IfRMz6g8XQ4XDQfI20+bT11yDdSvYnWrvtvzdH/CT4t67b0UhZKQKneaktIqATj4vTIAFHg76L+RCVPpL2LD5YLTSAm689R48uGsvanEbDRI7NayYAmCDpAmEEueu9314nnZERJGLwaEMPJ2Kx4ISG9XwX1f77hZ12AnLmX3uqBYej8b3b39sG2rzi7bAAa/VUimUtfvXvfQv8Mwnn2LxkGsIUUbAymPkOABdMmmKE858Psr9Y3ikMY0rXnwZpsbHsXHzFnzn+i9isDyAxRCYojYrM2B3bIp21EQh5LFsAZpRE40kknvlBGveY7vdtJZwztbNZTVFVKd1c6Q6Q46H7vvDfsGdL10uI077C16+xEnRV6T/8StfxgMPPGoYfKOpAf2CU8MQ737Da3DcxoN79oyVZ81iJLj/3tt12jE5Y9wbGvTnqE9qiswVcffObdg6OYcmkS4e40VtijqIOHyJ6ZXNf3CsXetatSKFaWmxwDHqqYQnxorr+KG14EZbaiyKPqaqHUu+hbyOXtFcHfbQpQl02CCPAUkTneTU3z+EQqmgMXC8xvzUAh668x489tBD6Bvsx1fe93eu/85Gu+hxCbeIim7m3yqgIU4+66XIlSq4c3o7XvXyy9FXqOCmG36CTjaDe2tTmFiYwkJ1CUnU1LNVin06P2igUtZz54KcKQAPbK5VUa0t6dACYhWe/MKAUCdq8339Ayb4/YKXIOmJWLVnl928+6k3g+IDfOTrX8KOfVNYYhM/o/OGjfwuVUpIW21886PvWw4endYbVSrFI/ffaV2jYYDhwiCWwggP7d6N+3ftA6e9WD5uQ5DIfy+VCAtnNJmKJj5fsgHLImW6IUd8vU6iEiOVymzRr6ZDaDqIjUenQDz/j/dLS6Hed3fsyMLCnH6m1WAA55s0+R4e1yZ2TmQmv6/cZ0WifF6t2SPFPE47chPWFAjqOJaP8n8P2bq9n6Z40jlXIFcawKONaVx26aX49fd+gioifPeeW7Bv9x4020ZWpZvUHB1X32DbOT9P5wNx+geha83+56idpmYOCH3V8CgrK9OtqavIC753Vy6nKlbrPfBrP1oRgEen9uKr3/sBduzYY5F1DC1UpVREI47w7fdfi4JGoi9/+c979IE/ycT+6qGHMKHZM/TpHbFMleY5/0QjQ65dsdBnlOwMO3nKBssqYjWfyvr7gU0P2YxtDsKzur6iXYNzaX2kyc70coPZWbBkFBV0BIv8uwNFOFmDMDXblnTEaLVuWLhmJLlBDBqz2gKZBfTJlXweh60exbFrVqLAw/6kOZbOMoA97vRLMTK2FvfM7MSHrrsO1/3j+/GlX/0YtWZDKHwjsvI3mU1SRTe7lm3q/L2OSHcDE2z2OQcgG3pJ39/f168z6Q2Asna2ZcH7kqXPT33x/8+jvP1KpMKtA+CaT38Ke3btpeHRTbTqdRtRlglx1MEH4QNXXWlND1phnuGQw9bJCXzlxp+iqeF/Hevf1rFlxqnTgmesLas6vyDghydcqFhCwZfLNoudqKF65G2gAdeVAmabcRe75sGDPNpEwjZrQ76g+eHlXj3l+SFkJvmz74ilC+Ln8h54f7wWByl3hxvFdlIlf6fqFzLa/DwpQlF8QgIErVAWmw8aw6lrV2GIz1EM0LfqRJxw8tn4rx33497f3or8oavQzmawZ99eo7g166jyUEhWNDXg0CZue1STsuY9ERX1ZW9aAI6Cp1vSc/oBlAzAKfyuqfeIneOieTLhfrNJnML65gCvv2EnxTv/9bOYX1jA7CzPRcloECJbq3gWXV9fP77y3ncgdLXoWpDBh7/2VdQ4NiUb6oiQYp6dtBS0+T0yham97FtX0NbuoJ9DgrKmvS3Oi1NbtO1gTXB2x4F6mhf9Hx9SftpNxTTiAidulG0sunwfq3vmq42Ry7P1LD6Ym511J1waLz+roo65EgqFFoAADg/3NdNvk78ZTXOEO6d1G1hlYA/LKszzmYszRz9qzTqcccTxeMa5z8Efdj+EY9cdii/9/scKPHfuG5eb4eeIE9COxGWk4EV2FW3dOo/ov2klaUH4HDq/p5BDP1FOziEin4BuK3KnZfYKXubCC77Ht/cGdDJSPTVzL/x//+1NuPnuO7F376QO/SHPnmANtY+jxZ9x+ql4yYXn4+a778FP7r5LTY8WgNnid32tZ+BqegPPb8/qYfg1Nz+HFStW6Pw5G49mw5asvNvRYpG5qwEA7nwZ1eXdDHrz3bQgoYY38ShuGzHuJli6oNAPHKBPlabHHeXMS9Vqd3gSNwCFwvIsn4MFG97nAlubq1U7FoSVNzfixRNMbWRMoHHnNKp8xv7KIC48/VyklTwuOP0sfPOOG/HE9m1CKcW2nZ1HvVF3/YghWi2jsrE3kW5LVDNOJGvUVSuxCdaWnjZ9+uh6+voqA0a+3E/wPbTh/yuo289fU1vCEFd/4iNYWKhpGjUVkBOyeAulgQEcvPFgXHjaSfjp7XeI8EfByyfnKNiiLkchtohLZ0JVzTS/3REofSbAYI+WwOY4WRrlhwaYZtu5NLxml11K4Wv+KwVIjbWAVZ29jrTou2jNh7puWneqhI/CuxbB8d1keplpMDPgKRsayWra1p3ooTMAjEfohyiYh7comxuBFUaCUayzX/6Cv8SetIaZ+TnxG7Zu3ar8XE0scYLq3LxNv2KwFxEws1OuRGyRGyNPYXkursrD6mewdjVuECrGsuD/jDpki9OFcntKH12hH3CI3ds/+0k0GhGmpucVPTZqNtRIc2Q3HaJhwjR/vDGdZknBMmcv8EhR81MUCjXMTmCsKHCisBgQSUhu5IiaHbN8COIFLX2n2aW7oK/lG1ivl58OQplgnbjhzJ4f70n3wSDJV+Z4v0pFdUJH3tqomVE4lyKAhNTuXM4CLlLIXYaijdeBzDADRDJ2+Dn8PSNsfbabK8DTJ7wbsvGwsY5Uo5AGDlqJJ537FGzfuk2pGcvNtCzjeyeQNFpoVGvabETl+Kw8a0mhk07T4vApy9U968jGwtrBg1AtweXxCmj8cVVdyrCDGLuTMRzdYZmdIF/TuzE+8fWvYNvEBKrVprB7Tmmy82dC9K8YxvCYnaXOPFrRdKXs8GRrCOC1Cjx1SVagoKofTaHamkJju1aKRQmRm4BmmMGUmgl0Ph5HtFD4oSJdHlIoQTnrQAvgF0QWhgER74dkkBxHtFkwyCyDGtls8v1sTc7oc9hDoPo5aeWlopWRHW9QAx8IALmxo1xs/seBDxQar6l5QI48yvunm2H0L1eSy8taaAN0Yqw6ZB2m5+ew9uB1WGpaUBrX21iam0dSb2tsvHx+HOu93IA2JdQsmT/3zub4s0GEOAnn+TuuwYP3/j61xTlghu2BPt6pucesZQ16ulb473sefwxf/vH31DI9OTGHQr6o1Ee48+AAVh98sB1Nmg3VDcoGDGq0zLNj4vB1FDoXRvmyNCpAlnVoQqSOOSvf6o48UWzSPQrMDiCgNjJgZDWQfycSSC1TuYSU8EpFAxa0UI4M4vv7/WYmMEQLQjfB82vM1Gd1xKgd48n4wE6I4t8NCzALofiGpedm0xpINIPVrAFfTyvjLSqxczWNJrZxma61kxiHHnOEaF08XbJEhm0mr3N2o0ZLhwtatZAwuKdpG+1a13Xt0lZwshGwJjNXabz/7t9Zde4AjfcVq16N9ibeC/9AwXOo39s+8SE0mxEWF8m1ywp21TSMXBajBx2E0dFRTM1OyXxT+NTu4eFhV+hIBXuWSzbtsdJX0QBFLThLkO7kDC8gj35ZfMB0y7c5G8uFAxm8hov5oxOiLGswHpoFexFTsB5yKV/L+6vWaoKhFQsw/qDbopVgOhVzWBOjbaNPSQDq+TOmLgtWtAIUsqhSOm/Oavn6HV2PQxap8Uz1CELxWjOTU+gbHtIZczT9tbkFJM0I84uLQv40ccMxj72LcmLt1hv8rF/rVvIbgefsulnB9931X5pzR43vFayn/nZ/2fPDMqazHAf4zfC2f/4Y6jXOrKPW0RTxBApCjQkqgwMYW7VSJowaNzDQj3KlpIhVJyGHduKjR/WGhgal+eaKLKf2zQKeI0cky1MmqWl2HLdZCk260vwkoiuWHtq1fHRv8YGVNN0UrU6Mpbrl8JoL70AeDwFzc/HavE9/eII0iqddOl9NzNxo2NY7wOfz2D/vheZd13Puocv3Szgh0/n+OMYSz5yhu8uRjt5Gp2F8Bs3+cz32XHc9k6/xusppnLBAQ9DGjZ3pys8Njrr3Tzd3Bd+bpv1fgveVp672uw/+xNe/im3je9FuJViYZ4pT1BgzPiyPHx0ZW4EWz1UNM+Kr0ReroNOJugQNLqhP88zk53XiIjeLD4i48GZuE12b16FGWquz5eMKLFmo0Gxao3Ornq2UyooXFA4hT9LH5LPJSyfzRXPeeVaeTZ82KNfq3/LVDgWTmddxIxaUskjDz5J7IP2cfATm7AUSSjtyORQmT6xmcEaloPnX3D926XJjRG1Zvdm5eRFccwULUvkZjG98u7lMfc9Erl4l9WCZZh264FOm3R2lEtx3501/jsk6qEGvO+Dsdf27p8nwwL/fct+f8L1f/grNRlvCTHQSFGfR1+RnVq5eheHhEdGFS5Ui+ocGFeRRmymkpXpdUCwBlmqVg48NauTf+BrCrjqpmUOVNJ3aOPq95t80gEMMbCqXMSoM6vRQrVqdecx52w4r5rU85GuZQYQGMXIaAyJ7boQqwR9r6ba5fPzZ+2w+o9c+Rur8PWuVokS56ZtKK4k3MHhsNPRMrD5SOAzWuGGZxtWjJtrVpgpdeY0zIx7h5v8fkE15gft2NNERPMXKtZmL2+i+ZAn+J8FbU9//LvgDTQzR3XaY4m0f/QjaLaZACRYXaoJZmWpRUwZHhvXf+Pi4dn+pr4SRlWMStARcLGjB+DN/x8XwttyEb5G3bwsiBs28lILSyVGJ+V47KcOdwuQHIzmki8+loNH7Sofbe3/pDyrQcARC0pEBONwYLHeaqY9ccOioVu6wQglQgRpLp20dHMQgtMh6gMiFlvdzTDsF7wEm4QFRpBm+5CJG1RrWj41hvLooZJM8em5A9e/tJ0TDOnRWgM4vW+4eNsKHa6QgZtAF51IE997xn1aW9RvCHxLYE+Xv5+cFCu2/KbzPd7w+XP1PHxNyR3Ig/X3o2oxo+mmSy30VbQI+RK6YR2WoH6NjY1Ys6aKCnIJdslTLmUlh9K7rlg/P3zP9k5+LLWgSvu9MGzWLx6eyscOKIkaNtrZmi/7FPA1tdoyCMoEthuVz09Gy8JHVu8+TJxrN5dxex4rbgctadDcPT2NgOQeIm4NTudsRSoWi3BTNuoE+BiX7moHO8AlYX8igWmvg3GOOx9bHHkGLlb/hUUxWF9BkZuHaprgpmSlYCuomePAZVX20MSuaKJY4i6nYwUrYstJe8N1u1P9D8JYO7F+qPbCO8++33Iwbf3eLmB6cwVpvttRMuUTggSzb4WFpACtffYMDyBazGBoelpA0BsydskBSJk210jidHr188iMbH0mioKnnmTpK2RxWrTyWgosiuQsiiL5TlwvF8WFWvDEXwE0gi9ED7XKz80RMjVmlptPXu0FNis79MaQy5cu8dS2uAB/bZEL15hYUh2iKSKGoZ6LF8CdcEtvn9TIF+vkYm9eMYSxbxrZdu6U8737b2/CO970fLUcKFQGTpedSHpe/+FLsG9+nieIkYDTbCRaqDdQ7MaqLiwbwaPCT9fzbKBEneEvnTK99D1ovAbFX4/k6f0Cu9+8HCp6HF73tIx9EQ1BigrbTiqjVUV5PXj2FTAtAXln/cJ+IGMLdXQ+4hv0zHaLQchbNKzjiyRAO4aMrkOnvOe+eu52WhP6W9Wqhda58aahcRr/XEaU8Lk3om1kw/T3DyZvU5Mjyap2k6Q4Tcpi+LI8zb0a/srly1GZtnhangwxi5042ctiMAB99cxPpYAaetunm5pn1KiCfy+Ctf/VaHH/EGlz7/z6I6blFNYf84js34PmXX4HxxUWlnzwHgHLaeMgqvPkNV1j/gPy6I7XyKIG2O0/HWciY6SspaHrUAMG9t/0qVSDUtfUuRXP+vSfH685e9b7/QMH7rIAb4+d/+D1+cvNvEUWphh00G0SnClocbjyadZqrQl8RpQFjklCQtBIM3vh3wrvM8ZmG+d8pv9cJGHbwMXc19yyHJnJDETvQfdCMavKGQZTyvZq358azuZRMGAPsaFW6CnXwdlujWfHj2H07811CdHiBdx3i2jEbaJpm0XJUFxbtaBN37h7TNm4QnW1HbN5lE9xkwgYyWYxWivjsR9+PsFNHOw7wzre/B03Xa/jlz3waL3nNlWh3mE1YZsHPf8HzzsUZZ5ze03NvG2B54ANPgmSvH/sarC5BjZflvOePFLztIPtyw/APTODdMZm9Qtfe2a/pwjj3PId23/g4PvGd7+pExHbckuAzjvLL06ZKRUP1hsaGke8rOnDFJmPzxpka0ZTTRZDRQj/JtI9HinNx5+dnBaHq9GWNPOF4VAI9OSFryvmzLO8yFfIgi82zITQqGNMFYvRc3ADcVLQAOvzXCZpuh75eR5u61Mn/TTUBx6admZ7pNjsYNsSAyyJ6uQimkJrQGQu4oiWjpVLzZbkfV5x/Fs6++BkIkizGJ/bhwx/6FBqMUfJ5vPTi5+Az//YdTdu01JDQc4APf+BqHd7EjmGnx12peSU0hWZgZ6VkUdoJtd/1+/9Ig2yha+o9r/5Auavo3zPHpTeN86aef6/Xq7pxfsjMUgOf/eEPVEsnlEmTT1x5lpMeuLitNjYduQUxazOu24MPRvNMn7V61SqlQdZTl2JgcEAIILVJp11ns1Z3dnwyXkSMWB5w3NVuRvochpix4z1d5G8Rrx18SOaFnbbp/L3O77RN7eff2IGExmSlv6fAVZRhwFZj14vx5ClwKYeCNxZebB4A/y03ALqrorQ8aEXIxsDo8BCe/8wzcfYzztPnXv+5L+G+ex9WF8xJxx+HxflF3PfYE66WwbMA2FxBwb9dNQwDgNxhB85S+yhMrogNopyOqfpEwXoO7rzphympyl00rqeTpjdt6BX8gZvCd4dw0hU1MQjtSBKal0/827cwtchTlFM0eVhRjuYt0YwXYs4Do0PYfMzhOqyI5lY+OZNRNWtsbMxKmSREzMyocEJzPjQ4iGLZXIUQOmnB/1fXm4DXfVbnvmtrS1vS1jxbnk0SOwOQwKEUuKec9gKnvbSXnsDtgdIUCJlnZ3A8xU7ixHYcGw+Z54lACCWkgRAgKVOB3lKmACEOGZx4HiRrnqWtfZ/fu761pdLnKk8e29LW3v////u+NbzrXe9C7stROh91Op7akJ1nLyRufEK/EykURSYVaURXnpFb8TTVo3zNmmCxEzAD7Ispl0zrrC7bkr0UvW7a0UK+IDgmsIbrYx481cLJoVHNigXIaW1stL/7vz5g7/3QX+geb7h+kx3vHlDf28qrr7aHHnzU3jx8xOlgVVXeJVyWsS2bV880Y85C7sTO+aPxa6E9MB0Azn+88LViZUN9iRY1G7HTwiew4D9tgj9e+cK0jYwO2ugINelxEf1cLqzCKusb7Ma77rGRsYIvvAK4aeuht34YgGTalp5xmoIh0Z1SHqqyLHRgTnN5ue19Y4+iZ1JBkDayALILXACBovrsRSzk9PrJ5k/eh0UQ2WIKfzzuQzAEAVeImSq/m8gbs0UXtVlIocYnrKWp2V7ZvVufB/jC6zWpuTTOnM3lAZUC1ERGrhD6Q3iXtYs/+yn78/f/iZ1z3lU2ylBirFxFhc1ra7G//av/0973Fx/Q765ccYMNDY1YRVW53XfHbXbeZVfa0PC4VWRJbSutOldtJ5+yxD591pkl9ywnrTx9RrHbvzczrox/w2FUeZuFr6irNQTw3E/8UZVuloz4fzH/kgKdtqGhfhvo7xHPjxMERCqQhViiaLbveJ89/Mx3bISceBoR43IbGhq1wd4BASInnn6KbxLkT5P6BOkPp5vFZNwZlGA4dt7hWnDWa6qzK3VT/bxCD9JFk7xQwmvUyiWSoSNaIHikaSq2AMeGzm7i2zvxwjti8bGHDx6SLw5M3a2fa8fOPumeGkZ5jFSuYOUVVXbRP37CPvahP7OxiTErL5bbhZessr7hwVJ9YF5Ls33yzI/a6e97l+bW3rr5DkG5bXPabOXyK+zK1dfZ1DT0NLIbh68/9ekzbemyJQmjjyFFDmyJZJkImRGTKRZTvJEKPL/8wVPFLHZfKdLMFzcwG579r7Ges1X7+o7bYH+fHkplzjFx57MnHRp2fzZjX//Bv9mLr79pY1PTIhYAWHQf6xad6MTTTlYO63VkR76Ae0XWmPaBQSwmChQUPKj4IaoEDWtyKs1uhWyQkCtRq9Vc4eVZOPgEU4Jkqd2X/LMDO0Q+QtuS/JlX2aZtoLfX5+6Me8SuOCBlDWqc1Ewel0VNp0YPlrEs+N6Vl11s/8cZp2mEKcdb6Np0mV142TXWOzis3ye1nN/eah//xF/bO05/p3372y/Yt771gjbF5ZddKM7ffQ89rnurylVZZXpOGzauKrVuz14b71FMGH6pVO3Bu+TZo9bw6399ugi6U54oxrFDSsWXPwJrwnxwUnqPd1tvbxf9jG7yknBh7K5Ib8SRs6Ld9rVvWtfggE1OeH38eNdxGx0ascVLT7BslUt0ccpFhkgsGnrU5CpFnypo2iVpFyYPd1JV7SPNggZFCkX0r0pdRc5pT4gsTnoBRpG5pmI6HKsKmrphnLbE7/Ue7ylV8XwGruvc6jDHeLGEoP2xKW1rqLV7d+2Q8jUz4tHpY2hh7A0sziWXr7KB4RFt3urKSmtvbbKPf/yjtuzUU2zTplutu3tAz2DjxnX2nef+xb79wve9M9bKpAmAZbxhw7ViA8emi8XWus2ur6TFn12QUVT/mx8/W8RsVtbVKZUKzvz/38ILiJiatKPHDtrxrmMOqGRhq4xbQ0OdR76iKGdUYXLyAtQp2LRlduODjwsRm6bXbmJK7wG/bu7bFjijNlPmkxdzHs0L8k1Yusw2hY8xoN5Kfb+6psZPU6RsjAdPzRK4GRZN8irqn/NNhO93yNZzfRDCgwcPeaahnzlHLZqrQwtIFbIUs0mnz/XX5RLmtLfZI7t2WFkmFW2o7lERTGij3KgqekW7YvkK6x+gszhj+YpKa21ttE984n/Zyacus3XrblR9o6q6zG7eeKNtu/V2e/XNvUpr2bCtrc1WXpGxdetXKo2L9Yrhi1E/iawrFrw0MQPYmcD3Nz95tshfsvnqmVGUs4oAsxUewhocPLDXBgd7rRZeO4CLUgLUJp3gr6JBSnV4qAzrpazJDp/IVtj6ux+08XEXIOrp6rburi72bhpGAAAgAElEQVQ75R2nWi5fJVpWTIuWdEcmK5WpoBITsU6NjothorKsumYq1FnDahJjSAOHiD0hhsQhWqRUL1eRZXLCTl12sv3+dy/p+zBo8dke3KWWyoT5RwnWT1XS403ZwalvW2wb1q6yGvAHZt8orYJXMCZ9v/8SBxeKduXVq6y/f0TpcS6btY62Vvvfn/yELT5hia1be4Ng7o//Px+z//7f/9SuX7fZDnV1C/cA76+rr7X/9t9Ot7/+m//pZUNflFKNI1SqWWjJzKT0TsLb9CUmjoIWXpEqIkJqNPgjiYlQdhbiNWl73nzd8hUAAVM6QbW1TIScLFXUWCzMLQ8eU6uHKdpUQWaNhzc2VbRVdz8iXzvQP2DDA4MKZIBvS0UWsPKJcUX2oH20PQnmRA8Gf54ia95P/w5lZvXDe4Qr3ZuE2omQmS3X3Ly+48fVri3oGWsSfjHQykRsEOkyNWzoz1Te5Tc+eebH7NOf+JiVic8fEqN+qpW3o10z2F9iNpWCQCvaimuusy4NcCK9q7B58+fY587+jO154y372teeUoFn545bRL9esXK9DQyOKACtq6nS2Jfzzj/b5syZ4zUTLdfMBogTrhOffhLiNbGh9TMWXgUH8B3pw/6RyH+KfNlBv3/pRWtpbVSwg4hIZUWVFgUkiTcLnhxBhEqjqp5VauFFa05pVKE4YdduvNsK9XWS7oSQSLfI0tNOSRRh5qP5o4oqXq7CdXNQfFQzQUrB4kaD9IirCN9NLd+LKR5TkB3wRZzgNKqssgmdBsq0iaemVm91nrjlkD0rFq2hps5uXLfWTjnxBCtOjNjE6JBNF9OoD6EiaeEpKKmBdEjmPsy8HnwmY2vW3mgHDxyVqa+qyFnHnFY755yz7Stf+arteeNNETm33rpBa3HJZVfbRKGo3L+utloLf926Vcm3J1WwpK9TMu+zOIhR7ZRf5z+58wzI3bNF/Bw0qap8zQwpD3CCFl8gycKk/fxnP7Y6nW5Mablm0kRtOJgutAHzoNVpGukDTQnw4NOAez3MwqRduXqrldXUWqEmp46b0aFRW3jCPB/Gm6pPXjIlGnWFKZogRGAYGxcaqNl3IVGCWeUI0cQwNq7UjxPeP9Dv7ohWbIE1nutrkzKIIE3OUPqTpETGoSinqdMANR9835/amiuvtPKi2ah634gbmLfjA5SC2RMBltDHXKWNDg1IRzdcJDgF6eimzV+wPa/vLZWYO+e027nnnmO7du6yvoERe9/732Wf+ew/2NDAiF199RoJOWBl6eVrbKy19etWWyEdDA9WnV41m41DZ66upyQL7ylfVCW18DwsdGkrq/PqWg2TwALRqPevP3zB5s1p18PioSslKjI9sqYEYPBv0LMQHyZ6la4MHHSkRRPY4cWNgl25ZqsNDY7ZZFJT/qu//JDt3vOGjQGkZKkbx8hxCi4geUNC0UT2EE3Z+XlAoZxexpqqmRLqUlKB4JRE+TR2vrc3BZ07DQtOOS9WT8BMgXbirJ115sftr//yz60yBAJxIakEy3Pxh+sNlVrcVOjigQPYTIwjYDaDi0RN5LZd99qvf/Vb/QYWcV7nHDv/gvNs88bNNjw2affct0uiDj/50U/t4UeeUNBLCkxgh4u9Yf0am549blWAES4v9QSIfTNLVj3a2tN8HFkGsHr+AnyKOSwkCQlFvoUJ+97zz9mC+XNLrUPUkTkdBG38Hg/K25jSlIbkU928uYq0s2UyOoFu7op2+bWbbHQUwWL3ids3X2vNjY32Vtcxu/OpbynIms4SKnncgUw65n1oYKjkNnhw1No5wQgmkwpiobzWjXIkMLzntJ4ZzPhgXTPbSySGgk1PeD0cw/+h95xhl1580cwpUtk+gTZJf4aYQSdM/p0W7TQYSBOoIVKaDfb3ei1cQaHzCCnFPvTQl+0nP/2Zfrc6l7M5nW32sb/9qN1//6M2VZi0u+7eqef58EOP249/8gvLVVWoXeqEE5fYqacttb/6q494FlOqqDocoRi7VF53/19q2UoFptikmV/99FktfCg1lFUjLwKJYdx+8MIL9rYl80oX7sAIxREP1hzzpuqWFpRJjZU0BjjJMVIfZ8b61CQPmKbsipWbbWh4TH6Mn9+983qr1M8mbaJQbhseecSmilkrpJ1LkYeawMjQqDN3ktwqAaLy81SM8I5ZFzwQ8yY0bpPbIOAsFZhgoKZIHez702eeaZ/827+xbMYBHW3eWXNrg7vnTYre8oQLCVPuuZUTPMrLM5rS4dCtT5f2RSmzJ77ydXv+hR/q3/nKKmtorLWLLj7brr9hs7W3t9qKa5dbTU2t7dh+u/3htf0im1SUZWzBwnl24UXnys/roCVwYAY2jgifR12wF1980d71rneVXIBboqQfHAuPaNAogVoNufekff/57+gimhpqZ/htSXXaETAvd0bO7IvvBZAwO5xULyrgGjwAVTm0vNwuu+Ym0Ydj4W/ftlYkTtiuba2tiop3fPmf7EAv4gRaAu3eqfEp61HBxrn0sF2EUSeeuQKxSCeT4qNOoEy8/8y7TxBKKLdcJmNn/93H7S//x59bVZXz54Xvp8jeEb0Z90c2EbFCtGPF5lIRKfUE4ttHhocS3Suwe8fSv/P8D+3Jrz5dGsXe3tZqly0/Rw0mdO+wyeEu7Npxjx093qvnVYuSRUOtrb3u2pIiJsGoW9YY5SJH6qQP/kucwzj1EeknU/+sOmlYNAYHEUA9/fRTdvLJJ+qGCXLYcW6yEidb0bJDnDxQmbBZYzuFf6dxozHvPRZDQVW2wi5cfr0NDbvCJH7ujm3rhANUotGiuyGarrSf/eFl+9Lz38O5+jUUnWHTfeyYn6BUD4/F8YDQF1dky5ioHLku+IKZzW9pspvWrLD2+nrvLk26PCI6pA5dPcA0GCk2gOP4bvaDCqZzLDVtmh99mANZiluWJJU+i7j6rz/9ud13/yMKRCGcNNbX2YpVl1p1dXQQZ8VfuG7NRhseG9ZmbKqrs6rqClu95pq0FgCSKY1TQhGMx1my6SVqmd8Hr9GhpUnzVz/9pky92o6GR+0H33vBFi5aIOozJru+Nu+88SLFjBk834WC3SRi1nkgihjl99ko3sHhgVROKZiozsCvmaxdsXJTCthM379n140qENH/Hu9DuZQHN5HJ2LV33O8AROo2IVXr6+3zjtxEeIgALiJcFt55Zj6bDbPN6Xpww3orKxu3wnSZGD+FIqVTb2TgofC8iBf4S2QE/AnCCWLnnD6PH/izpImfNOZgzzJwwQcl+eKE/Dob9Pe799jNm7eKOs4haG5usFWrL1fU7uaYg2V21fLrQEv0LNubm62uIW9nn/0PrgyKi0nxS3AHFUeAxaSNHHN3JLUOd5/ANU3+yPzyJ98octqBQr/1jaftnW8/Tdx1ghcWlO+HooKCiRTQOfFgZgge9fN5nXOVdsUpd7NeUSJMRmcKC3Xt2lu18Fw8alcP3rlRHHTyScAKoU78fuqfw7Uc7h22TffdZ4VMJbwTmxgfs5HjA15jV+UpzVwTugbxg66TolVDy8rmbH5tld26eb3oymEVwjopABRVimmODkBxjqJZg00nV5WYupoNk1IltzJZUchp1BSSmBpK/1OKpdebdR/rtWvW3KgaAYgc+fkN66+xyrx3DWsDT2ftokuvVhNmLpe1zvZWe/s7ltlf/MWf6RoEa6eqYty74whpzFnqsIkMzWv0qbmCLODn//rPRdifzz33rC07cYnVVNFYjyKEY+Z6gCB7oi27VruQqfSQ9drU5kSlie+7frw//JK/LRSsurrGwZVCwVasuUUiAgA1oH93blsnwqWbZg+c5NNTuTWTqbCqykSxKmZscHTSrrt5i40VfIePFt0X47OrMlmbP7fT1lxxvvD3J/7pafvO935gnS0tduut14t4ETlt+HK5nOq8TjUBGqdYFLCkJOHjv5JJTaFxIHv6fHoBFAzGwMQU1AmrD1DMad0T41N24WUrFOzyzBoaau2mDSstW5Hg4qLZm2/ut1u27rKKcsx/xpYsmGvLr7rEMpmC1iWYxbMnRUe6GJM9ZMmTJaahItyhNuxPn3+8+N3vvmCnnbo0MTxc4iNStWC3KlKW6pQL7Qgpc/6+m0janBOYQt+7QI00CpTXw58bEUyK6obZVWtvsf6BARVramvydt8dN2vufHkGnRifkEzs4PPnvDrn4zNnePQrV9xcaoxQWiWt16w1NtZZ59x2u+DCz+l7Tz3zHXvyqW/a/JZ6u+ULG8UbCHMoM5w2gqJvYbyJmyC1rcSizbqbixgioiosgtqjmQ+LsGAqAPlrneipDt00akVoopXZ2ede5oTMigprqK22LRuvs0yFxyZsqPvvfcx+8eJLum9g3faOZlu9ZoW08pIivehlIe8+E8DGjJ/AFhJHIG3agLgzG1aeXWxrb5NClSSzcg5IBMghdAzfLUDGNdD53ynGng55O5J3YuLPKQQoDYLsQJ1elkOgsDdNTE/blas3W08veDX4ed7u2L5edfuKLPECVsSDLKjOcdpwG8C/nmZlbPW1G0Wj1olSX7gLLpRnM7bkhAX2+c//g0zwd773Y3v4sSdtYWujrb95re41uGhebk3zWCPVic2VzL3nhCYNHv6OSS8FkOL50biAOINvmBIXY1ZziJtc6U1bMVNuZ597qTpmWNimurxt3XKDwciLrGjjTVtt3yFK3rRHl6mCt/a6lYp5mPghYCqGKSWmUaSVgqFnz6FN4JIsgdZryjIP3bamKJECpj4nJQf0UllwuO1cMN9n8UhznNPuu4jXxIWGuY/GhdmuwLMGtxLezZq1q1Zvse6efvW7N9fX2q6dN8qiUL/WZ03RxeradVLByniaKECoSGlx1G6+eZf14S6IVBWJ5xQYMQh44aK59pnPfkp0rkNHj9rv//CGnXbyMlu0uFN0anrl8MVsJty2UjivcWrhnPvuZVUWLJfzThgBPtqYbr4DyOHa3D07WBVBb4xOdTTZlbimy8rt3PMut1GqotmsNdbl7datN6q8LZ6AmV276iYbHByWBauryduczla78qpLne8fbVJp4UMggusrtYZhOXhuCUAS6kmwGdnFU49uKfJwpJScfGz4AoEwqTpFJEmRI3xiFEViZ4m6m7a6pLaS6A+vj4fA+7LBeGRXrtxkXT39+vu8jlbbtPFa3xjlDiCRiaoZMgkjwWzJV6NQ6WkJVmPj5tutq+t4+r0Ka2ioFyO1sanOOjpa7JOfOlNmloCLY4I1IXLOZXMCmlLeWLIirpU341pYBLF1vX6XXh8m3Is30eEzG0SLDRB6dv4MQ8QYQnTWLrz4KhtJHT51+UrbsWOTwKuQTrl6xY02xgiVsqzV19baR/7nn9uHPvxBT1Ol7emB9ezgkc/l50o92ZRcO+4mYfmy1jFo6smHNxWJ3Gvzdd6tAsslpSu6UwV6iOL693kQ0XzAQkTBgw8jOnfzk1QhJj3FC2mxMEGUVq9dt8WOdPWqy2XJwg5bv+Yq158LkaCCYwFkCyx+c2tLqWMmINC77njE9uzZ50ui4MXZMvnqnL3thIX2d5/8XzpR6MjA2OEhEUVzeh2EcuuFC/NbTQydNILUv+dMW9+MiC0kD6vx5kkpOymGJ6hA7ztTxp0hiWCqBABZwS6/Yr1TyOAVVOZs584bS5ItLOoFF6+wTJlr9rQ21tt1668pSbUQJM1G61iTCLi5ZpWpIYKAaqaRrtRdWAusreKsrzy0qYhpAjiRZKeK9y4XonRMunBJICDVvLEQ6lWnUpceXpjxvr4+q63NJ/66CRCKFEUdKdPTlq+qtKvXbLajiCRZxk5/x1LbeMNqO9blFGJF3DKvvjC4ABSZS+yeJIT81a88a7/4+a89709SnpA9GmvzMvX/++99DjubmSAM8851VlfVyE3lESdOSKMTKWPIQFK5VueJ067ollUDBUp1Sh+9UMXChPXDlJcoVknXPho6FOJp6GLGJqen7LLL19nwiAsmsJluv32jmEK8fnh4zK5ZeaO6Xri+jpZmW37VBdbYWJ+yJdq93QLp2SSOXUi6qlsoiUXF4k9Oem2hIFZQ0TLPPLHTYf3EEC09iFS/hdzoJ9bLmhL2Gxv3CY4CRvyUicqcfocLUJBFPp6CDPHjk3+hpLnu5tusq3vArDhuH/nIB+3sf/h76bROTjnOz0KJbDmbNJneV71ykwX70Q//zb713A9SC5F5kakwaTVVNbZkcYedfe5ZJb8dUzV0ipl7kNqQfAqVjLPex/vrPHMQbSyJL+kBaayIl6rDWkARE7CUBhGT+noeP0Nr1sZELpyYARZxttwuv+I6G8CHp8aQ23deL3CKNHLfgWO2+dbbdVX8bltrk61bd40GNrAxSB1j7h4Qt0u4eWVR1PJZqXb4eFwkhJviNHqAE5b55y/vKEpdKqlO8QbSR2WokJoVsq7QkM+rqUDyImmjBEZNYKWO0tR2hAsI9E3pA/1psQkSiLFq3a12+FiflZcV7NzzPmMf/NM/MXYlpd1SO1OKntX/HsP1Un9aVWXefvbvv7SvPPmML1sCLthnNZV5W7yo3c694LM2gFxYdbV67Fx0AMq2F410f0HhKqlJO3PWeXze9qTYJQ0+ZuEduHLLhDXxTCe1Zycp2IgVPNjDiqYp2slDL79yvQJTMY4yGXv04S/YxCgzP8yefe5f7BvPfV/3xeZfvGiBnXvO3wvoYWGVVeF6RVObae2KjVLadLq+mfmBauWachmXzDNP7tJ9STSf+6P5AHpUak3izSXMM6szQ3LiibvNRXDS/cykScVRjEmSXlgETqmiYtKJyQnbcMtdduhIt0zW+uuusCXz5uk9AJMUF9Q4kBTyJ3yPVqXmlhaJKtRW5+3F37xsDz/6pCYS4YmVhmbM8tWVtnjRXDv/ws9pEfF3LDqxjNIwtRNFFO4+XlIkImqSK3ljI6cJV0Yc4q1UTufyeAewKXHVWeyyjDZXTY2TUBzV45ky9mw2G9aVsq66+gY7drxHz5Hq0UP3bnFpNdi1W3bZwf2HBSXn8zn7m49+2P7sgx/QhA8xmypcFSwieFqp9T4zd1WCk9lwMUJFC53EETL//JVdRS+0ZA3/jE9nN4cEiSDNFO0TaHHyWTy1IScqNLtesqOSFnXmZwnqTREP5ghUTOlexuy6m3bZocNdetB33r7ZMgValLPSveXhYvKxHIj3ElOw87kWsgvy6FxFue3dd8juuONhMVcjd6anLJ+vtPlz2+wfP/spvScPRi3XqeUZEMjTTp9Dq02dsIMo7tCdwzw4ZStpfrteA0aRhvTOLnzAk/PBQNTlgZvDgzoJNMxvIgnZqlUbNe81AuqH7tta6nK94sr1nl4WM1ZTW2nXrb7GqvMMJUjCy5p26WNbWUzkY4LVzLrwjAKMinm6cnFYsDQFK/PNf7pLZd3x0RHh7J0dc7SoAcWyMCxqgPwK4ngoY+jI5RxXTjVn2C+8nofKe0SKp0i7psb6epHppJW5zDZsucv27ieYm7Z7d22x0VHXguVzaY863tWtMnFbe6tj0gUX7yNvlpVJzYq3bnvEo/FS9cuspjpnC+Z22OfPPat0+jhJdOnILKv44+6BgI2TpDRITSGkfIg4OOvWT6+3OuHyAgQhaJVaRsbUYRvQKe8fVObIhlIQUar9Y1k23LTd9h44oh9hrR6+f5sXfjIZu+SS1Z6wZZBmr7atW9bLGmDXBBOnnr3gAgwMuhvz4pLrB0iBi6JNqilEql1iCX376/cWCWIYBshDr6eBsqxMZkunOBEWuUBSIXwtUOv8BfPVBaN8PeXamobADhwaKvlOHrgmH/NwKirE3CG6WnfzLtu3H8Jh0e697RYbGOwRT46NEf1uLmrkSo35KsfxNWAHiLSsTDoyW7c/Unp4oZbFaxfOa7eLLz1P2EOASogQuniiq2ViNuvqanXvwdlHWw8zEOLE9Oi3d3R446OkQV0xm9erkjcrBhD1WzJrnh56U8esQFFyJCCgGbvzrkft57/6rbue4rRx4r3nLmMXXrhSXAGRMatz9oVbb/BYIJl0hiV7FuLWhdgLy8VnKT7JmA3098t60mAZBaUA0aTg8fSXdxRJCWCv8tBZIE5+Hb3n2awWW8EWQgac9sqcbhqzjWaqWogSpTp2VcmspGmVIUYUYANuZMuO++2NvfsE2Ny49nKrqnJFDCL+uXPnWm9vt/h9mHuiUTBqmgoamMhUkbPjfT3Syt207eFSJOtgDx0nRevsbLeLL/mcyq0jzMqh0saJ1agSBBRzSblaOtNKrSR/htCR3FZE9TktOm3bbAoWU0JNqUGzVPhI9GtMKbUGzC/uM0rWOqmSP4XoMWZfeuIb9qOf/ruXbqen7aEHtrklmyjapcvXlizVkiVzbMVVl800iRDHJFfiwxbR05mWRWVD8qxiQ7ju3ozsCwuuRhA+876dq4twzcnvhoaGdcNNzc06ZWwAgistSNJiV2SMhPew5/IaQq+pkS4jovp1ivypPGGuBQer6lXU6afosGn73bb3wCGhads2rrL6hjrr7e21fGVOFqOmNq9AL4KRfB5LwAiQvC8SsmeZrF2/8Z6S7lygisQQcNXPOedT/6mowoNtaW627u4ebQQWX0UgJMxSB02oWChQUq48Q1dSeprN6p7AFbAexD3yqakti4VXL37aOPLvCXbmT8Ajspenn/kXe/bbz/v7F6bt/vu2CBc43jVoN2zc7nX5TMbOOutMe/97353qFR6QBtaRiEkJeaSJM5uGFVBPcJcY/IzI+wPFyzz12Db9fn9vr8y6JjAg3znOhMcaO9bVJRlSpQCa4JzznF18cadWCRiQP0Hsl8DLBXOl9ZYqfT7IB7/j+ey22x+w/QeOyjzt2LTWxidHxbEnIg+aFO+Zr8qnaNwnV/GAWbDJKd/dW3Y85sIJjhK577aiLVzQaeedd1YJU/fqmJ8WeAEekfsQhND04b5C3YprwISWxpmkBRQ5RYOKvFAliXBhDQm/T/AoboUrIThlc7Q2Nycl7kptjH/53r/Z40885fWfqWm7686bREP/2X/81h770lNpgTN2w/oV1tpSn4gkXq8I0Cj8tQLKcDnJCmhRU2XQM4yUgUiZI2OZB3etLerBpeCovb1dN0KgI5Rpako36qXHENrznBRhQt6UBSDCZcE1hVGRI6ifpxj45SjiuBLkuH35q8/Y7lf32vve/z778J+9x6oqMtZY16AuU8zf8PCAhuqRaYj1guhPmhwtl0JaODFht+583KN1wff+8Cn0zJvbYuee849Q9EvmNkgkWB+v4nl/XnXeCzDE6ywms2DYqPj56LSJdEnVskSAkB+PPJ6MRhp7KHcXrLbOhxPFEEDh/lOTcplcx+4/7LG77nncpssgik7bPbdvsInRcXvya9+2X/92t1c1c1m7bftNNlmYSDAwFctE7kzgTqCGKhKBpSRsIhBV35z+O5HWsUkyD912XRHzLT+O8lQFPnFE9XNyeRoAJEeKxnxlpcuGxulJ/eE8DFA9ImF0aWQFCtOucjHpUqUsDnGBFC6nRq2vf8TaOxdY30CftTfVCFQhnqDsSO86Pp8ty4WrgVEzU53gqdoCM2anp+yW7V/0DpkUvbLwbLh5c1vtwgvOFo8vGLNcC58fU5s0OEnux+VRsVDcBxMmws9z35SbOT16JggQp4kVGvaX5MSoafDePAusppetedppmEHiDDJlA637w0d6bOftD9oU7RKT03b7jvVS6F69dpONT7lJrygv2vatN6R+f2/R5n0JgiNeioYJXi8cgdgs2Eiix3n9QdZ4zGf/lhY+UjcJC6RZK/yd00+jfnDleEgENvh+HiILSbDFG9bV15dwb3xgCPFhmicm0wAclXLZOFM2MubBGgFJU3OTTU2OiWpMoSYw+YgHuCmkTzipOvkEZpzOyQnbftvjdrynr+QTxQ0sy9rCBR12ySXnCgZmU3M/nFriEs19b2jQQ+F/dbjU1np9IbFWgEVZaH4Gd48NpbI0zBxqGmk2nvDxVP8Omhgug0AQcYM4iQR86v2bnNR99A0M2+atd4uUQaq665bVet+r19wiS8RXS0utrVtzpahXDh+7mw12b4A4ZCkREwQaCVfC3WKlN7Jq5NqsqdrPffUOVec4NQFfhnnG1LHzAUwI+PhApSipVs3rWfyYDs2Hs+gsGD8bGurTQ6mqIlAb14Ai3gPW7vAI05XGRSnm9zEenDhOPBRlqURD5EReTGM33GSz8SR4hFTY+Jjd++DX7fCRLl+wZOoJ+uZ2ttglF39eboVNiG4OqRnRb2AToYQp7kDykTz8GDEWuTndujR8Ks+vdNWNqJtjXsPPqwyaKnnyqXQRkTqlmrhKpQwsmJy0o929tnX7/TYOUlqctju2rpE41OobvpCGIJudddbH7U//5FTxECOg00ZKuLzirtR6Hd8PX88aB4jm2ZZDz7FBMvfvWF3kwXsfe4UEh/bu3VuqrXNC+CgX7Eecr0IkR+XmExMym1oYhuPy2oxDl/y7KhUrOHWcMjVCVFRYXUOj97mn2vHSk06yPa+9qt1Zm3dql5vgKQESwqaTADEwRvTb4wLuuvdLtnf/4cBIPPjJZmxOe6tdcP5nk0q1qzlSl48TyGIp2k4Vx4CTQ1YV7r6gaYIEPThXsI7R4qBqLL4zV71FWhi+mLVeB/DeA7cibOYgdvT199r4ZNHWb75H/Yll0wXbvmmVmiCu23CHW5NCwbZsWmkNDXnXmJ+loKl4JPl6ucLUnuYTrD2IizQzYgBxJmdRvDNPPri5qFku5eVKdfBv+HR8ReSyfIh058fGramxUZOeQwUa0p/06Kp9Hhw3J6nS2tpSJwkVM77UKl1drWIOvppNIOVo2rAy5s2WVJGkLJkGBwFiJFCH08r4Ut/97p+/+8L/az/6yb8nUoSbMtK5OR2ttnrVlUltclJsov6BvpIrkwImLqC83A4dPmxnnNp7wtEAACAASURBVHGG7d+/P20cFzyk946v0RGkWP1gEHuoOFNI/HQtEtVIL/mCZsIeHh52EAslbmfwuGz5wADACmXhCVt5/Q4bROuvttZWX3WehgJuuOU+cRd57Y5ta62y0q2Gl3T91AaHD0EJAl9POJ14QeMr68kaIBUzu1gWLl2bgRMvOHNyUmkbAR1ADr6NXYOf53TqgZaViTwQ/5bWfEKmODm8BwEOE3m8uodvn3bwowbhYpSsahXxk+ZJ7EjtVhU2PTGu08PvifWik+vTJAI0UmtSBbDujMn68b/92p57/kczJAaB4UXraGu2Sy75vD7PpUhclQq0TeBTZaUNj7hvx2+KXZvJqO88AlG+R8Ap8inFGXwmQ4/QpZ10N8hmlYpXb59iFhhZfhp9ALCSTJlnL37JGihtnLDBgSERSYDAW1oarLd/xB59/DkFfOUZAr4NUr8oSxp7bDanpSW9H03PxAV54ciD7jRRUi7HSTQ6uMz7FZTr5eLMfdtXleRRiBbZaSw8lTAwc0w/1TAV+4FjBweFZXMDkiVFA25iwos2lZVqbyIXl79XLd/noHkg4mpSfuK9i4SNxe4c6utRkIf16Dp2TA+VGKMhjSP3ua/MdEWe2xEoLPBrew7ZV772zRmdPh500ayjvcWuXH6BTtro6LATRhIW7s0gBUXz3G/QpOMABOIWFoyUTGmZ6tmetlIdYFOxpG45/MTTg8c3WVjPnRl4QDXPMx9VNUPjvrzcjh3rsjGJPUyoU+bbz/+HvfTSK/aRD73f3v3OU0QjYw1k/pNiFfcUMKxKsEm2XDSwtLDMo5UGf5KlgTIewZ024z3brlV1TunMLMIgb6CHklgoBDTHjh3TYvE/pp5Ai0XjxLCz0GZXBC1JFMAPj045FZ6XVgl1Q+mivqFBwAbvAZefzhOsA12vnqZHH56f+Gw5phKs3LONnj4Yuhl75fU99qXHv1k6WREftLe32PLLztECtLd1iIeeS+NJXRfeewTpVcM/e7nWI2fSWSwULof75+HREsU4NJ4JQR6bxxnIfqLk+niPSUaCIVPuvQUQKLkmCUgkBlBg5vw+vQVo93FwYNmyOZmRg0VkA7uCd073jJXSGqVpWQHKDDN5S82sHrkHTyAkVbFkfb390jQQykpQeN8XVhYx35yuzrlzZWZZdD6YD+MEYqoxf0TGXCw3HmYrAhHMF5EvEiOcJAKjU0492d58881SH93AgOf1gXpFqzVtUJXykc6yZUEEqkwVrLW1xWe0ChFz009f/sDQoBb7SHePPfjAP5U2bUT3bW3NdulFn1WRgnQHISbwcyhU1Arw+ceOHUkyKv4wdBKS+dRg4YTK8Z6cZMQQCSxZUdI9CjwgvnJxQ0OOeoIjqObgVCf+HXT1oHFFNsFocg5DSTE8658xMjik9+BZzu3stOPHfXgTh0ULCzO5qVkHyOH0mVZtguFjR49plDmvDT4DUARunH/LJRDccWGcxDid8m1J/owXeTQ641cJHjgZHrABsLgfA3L1TkbHwStSmRUxA7B9Bg9wOggOxfhJKhli8PYOyL3gJubPX2D79r2pDbZg/nxh+MyKdxi5rtRdg9sYGR23W7c9YNAdImJnYdpbWuyiiz5tSKgA7iDAFOihIngsVlVOkKoIGIksIi4BSGZCwaSsmUrN+M8RMpqEjjk66vKnWBB6+FlUucBJ9HtqJYIk0Qj6DhNFjSd0YP8+65jToc0caJuzoMo0WkxoZOpNJMbk2rE+nOLWlhbda1hp0kDoYiIfS7K0zMYmvVTMQivwm0hzcxltysF94el7JXdGHo854oHwIVwEJx3zQIAjCDeZsxICVlvrKRraqtTgB4c89ROdyCxXRdsvc9Rm0g8eIgUZ3pub6JzbaYcPHxblGdmSpoZ6uQAsgEaI5SpcqjQ1OdCGFZuQGxoZG7ONm+8RgdHXwQmN7a2ttuLq88TH91nvHpNgTQBWlixZbAf27XV+HTBKmoAVhSQ2PPfOtej+E2DlwxfGSj0Hk+PumvDjoHYcCLlITYigquh+nWMp/AN6mmhkMSTIRBQR2AKqpgDQZ9UyVNC5fd74qSJPYvByaDra2/UssjR8pp5G75fM2uDIoAJ0GEu8J8yg8P8K7p56dGuR3Xrw4EEFVbX5Gk89in7jbAahXgzOZUGSXjy5Ovw4bi4qeMh0RXTP08BN6LSOky56kMNO5f3EdFFXicmcHT18RClQfW2dNOr5u/rFxz0VjNSPhyrAKIk0DY2O2LYvPCwlTPl350xaW3OjXXLp5xL0C7fcIV83s2U66SCF1dV5BYq4MaJ8KWwB4mBdamt9DnwaJYaPnanJ039OwJeIIeOjOvW8P/eIi+G1ZAFh2hXYJa4cr+FeuGZ+TvosskearsWfHEYWaWCwX+VpuI3CM1IbN88QYE15PYcSVDFN04TQGV1OakIt82oi5FAJPN+86vNFOmcOHTzo82KYA0NAQ15NLp9oVujEUzBhARSoaMqykxV5oF7R86Apeu/YYa5ekZFPOnrsiCJUvtfb22Mtra1aALIJ/BI3m2d6hUZhT1hn51zrp6M2je12IMSHApHH8/6UZ9ffsMuZp5hCFSMKWvgVKy5W0aeqslqdfDKfAmO85RndOFJMABBNhEIFKxVgSgBIykBYRH4XtxTxgIK0NJYb2RPuq4Q5CIhCQNEbNORXVW+fKEHEXIkvSnD1/f5kuczJFHKnBReVAtlUgJjyMKXS4hk6stfY3KTAT2BRUvEkm2FThJoZ8ZU4AET1BDKB3ukkFoulQobSq64ulWgx2dJwTaO6XfKjwnJV1TJN1My5cTYIX5HqiVLMOPGmJlmI+JnAG7FyauzwYachQcLg88gI2CREvexyfhfaFXPaBSyl5kJYpFu/8ID0dOS7U8Nlc1O9rVp5hbRfVTYuEJn7MILpwqQCJzIJAKnxca9gaQa96vAuPe4pqVfyWHhlJpWVCb93AcV8jc/VQ+SRe4Eyxu91dnbIiioDSkicov3ETYiN5fyGGfkYZQjQvVKgyXNVYSilnd6945E7VoKNxJcXrmpLimOIWJGFsFayPFUuRhl9jZk7brlKvXOc4qVLl9qBAwf0oMLH4X+5ccyc+wrGfo4IPaJCJohUzQZAlFnNQeUC2MWcgCA6AA719/dpNxK88OVRuqNOXKBvnhrr7JxjXV3H3IRly23JkiXCErhZFonNyBefic/dvOUeG5GQkpyH3qupqd7Wrr7SpqbG1aXLPSxatFjz7tiIPgfOu02HBgls/RipxQsRzHRCuTpew73weQ445YTq4fqQceX7lRWeQxPn8Bp8O6cZ9IyDwCbms0WuTPPwuKbgJuo5UuwhSE7TtLQOafCwIOxU4FETaUqT+VMVRBXDnOrFe9U3Nsq18vmaZJ3z554HUcUdPbBzjRQxyLV5QVSywgfVCfmCkzeskRqqX1d72bWxqVFMj4qqKkGRLc0tQvZiDCe4tZdEvcGClIyM4KSlJ9rhQ4dV8QIQUt2aGfSCdGlxctIlG6Cnpzfx5MgGhtEjVhwRp3B0ZMx23v6Q9Q8RiYsCJ1OPysT2bTeL0/fWWwRxXtIFTSTadnSNBgrH1MmDfeNxj6N6+N6gUVBXb6RGkQcPDwwoiub1vA4iJCDT5Dg8QUfHQjc/3AfPhoWJqppQP4KytBmi2zbiBJ4dC8e/OZgKvtM4E0G4QuSmZCUJ5KIoo98vK7P58+cp8GSj5MBfqiqtd2DA0+aHdq1V349gypERW7xkiXYoH8omqKmu1oPioXd0tCvoIjjgZKjzVcN33Q8TQfN9plRwwVTj8OXKy1nQqry+DyCxZ88emWzmx0RDJic5YFz3847wMYMWc8rNNja3lJo3dfNl5bZ9xwN2uKvXyQoSMTQt/FXLL1B2wIZgOLBSoFT544EQvPo0rH4bGhoUYKLMJevSIdFBrJsjJUq8BKGOlRVyFzx8Veum3NVMjsFBdHcZiCDP8Y9TSd7P9fm8cYUTC/dBAdnUlDaUroHa+6zysdLrRF5l4/D5mH5QVoLzUO5g4XHPXJMscHlWaOgodDYi/3u3XVsEg8YUs2vmz5tnBw4c9FNAwMaAPem1wsVjisSw+1EK/0PEBjXin/NQTznlND0g1J727d9X0ogFHQPpqqqu0ebp6u4qQbPQmzw4rJArwG9pU6UCDuYKCyAs3YpWla8tVZ686FBhd979mO0/1OWroxJrRgu//PLzFXfwu+IMjk/IauH7sFyaDZOrUPZARTIfRJM02I+NxP+AM2wIOAccCj3MfLVP1NB0aDKAvHrfNB9+2qN1FW1SSsufvJ50j4yIwJb3xcosXLhQCKiyIyZWzJ0rF8DPgvdIhM+z4ftYBtaM9+HeOHykbaScvBfumc+m7q9CESqflWzwPuvonOPj2+/ccrWoV1wYaBbzVkgdADHYfZwI9a2rQW/Cautq7Pjxbgcp1EAxba3tbfqgBQsWKdh4Y88eFTuOHDooszw27sI7oF7sUuriUaliUZubW3SiOflAsTwAuO64noiS+Tz52dS3xg25WZ60+x940vbsO5gWHuyaIQaNdv26a7QoAEbsekAkHzgMT5CT4DFKvrbaDhw8YFUpwuZ7nDYHZWDo+hcnU6kX7WRj4x58DvQpI8iD4jHQgGKMmlK8hZnTzmcr4E0NmNQ6cA9YPT6H585z4b6BxTnFfAbIHlYp6FZ8NoeR9YELGVQyFj6wF/7OBuN5UW3kT/7NpuU91QcJzsLCk7bh8BU9TkyKY0dAwwvZUUqAKP8Jqhy1uroal+lqblVRprwypwAMTdr9Bw4odyf9Q/bTOZBOoYrgiL9zs9w0sDCvJwBbtHCRHTh8SNaAYKmXacpJDIFNwyaorW9Q1B9AEzoCTz/zPfvliy95mqfGTZMcyoqrL07TrEflQg4c2K8HXFvr0Ce+kWvp7nUixwAQKrl6UgHhZHGSCHjD9NfXU2MYkHii/Pi0y6SjOQdbloVXrp1m6bCQPF/undezCByCUPrgOfzud7+zBQsW6FnPnz9fr6V3QSc1MaJwURS9+OJ1In3W0z3r2YQDaTmBTcIGxh0yZkNw0gX+5HL23ve+1379619bZsu6C4oEZUCP+CwWFFRNAgIELUmNkg/yC3YVB6/aHbXGhkZbcuIJYsP88ze+obo2P+fimhubBLm+/oeXtePnzJ3ndeK2NkXtdXWgdAM68ShO8XB5aCwOzX0e3abOWRWHYOb4BGeEijiNVblK+9mvfmfPfOP7LiuuWINWq1q74pJzlCU49s/UKm8I5YuNRHDpKaW3j+VpkEilUzYAnT/4YQ1CTNOriYNA2PgdlULTtKmY8Z4rc4YyMDCmVmlwKnhFFB9FG5nuoSGdcmIfPjMCOw4SGEfEFqxFYChYTDYk+sNSJEupM5uGU87mYkPx5VIxno3xfKlUCrm7beMVRXWKpKiWF7vSlHetjAwNe5cpxY3UKDk6NqICBf6VEmVXT7ebqrq6ks/B17zx2uu2aNEi6zp8QAtOVK+IHV6czJM3aipTqHH/xRc7GdE/brC+vtF3bOpmxdqoKpZQLJC+3a+/Zffc94SnYEp1WPgaO//zn9am6uvrtWUnL7O+fvrwHH3ErXCyiFmGR3zYMf0vge4pVshmlbLxoFg0ngMPlX+THeCKGuvqU97tDJ3pCWrt1Md94pboWKl3TmlYCqSxKirjJiYQ78l990GBIzDDNaFUUkWxaqbeLiJnoWDHu7ttlIENCbPn+fNe2igJ/Yu/x/eV7ma8Uph59I71iuoxXYJqCVwgJPb3loR5hwaH/lPbNDm8LECuPOXUTvUhuuehMsWZhwKGT7GGUFC4dch0UCiYnrZFixcrTeRm65qa/T114jw7EFN3xDdepEDUrQnIGpo8P+W9D3X12l13f9EFHBLwAfNlw4YV1tfnwBInWxTwXKVONy6GB0KARCmY6BkiZXtHux3Yu89bk2ZF3XFqA6lkk6qZos6DUfRllXINDft9oGeT3Bvv5QIJ7vOVMZGTj4zIDQR0G3FMUNtb2to9xUaGvabG2tpaUg9jTgeJg8nPAbckHZtIGuSZpGz+5RtKI1nT9agY9MW7bxQDh2I+vp03Y4FIT6Sn1tMrvx4dMyw6YAonulDEV8OQpeFwyoZh7wD0JNVHTKxGh4F5T3jk76bc+fhcKEFOV1e3zV20yF5/7TVra2lNPpLFB+BgFq0PG3D2al4na2IqjdwqFm1wrGDbdz7glOM0mQGLtOLai8TKxczjUvbt22fz5813AEO9Zk5oyDGWVFQpD8gIpvCVjkm4v44giWcDs1gyY2lapSt8AvBM6V4HBgZF/Y7TzObGYp104ol28JCPMvMEpCjAiwBOzzxZADbHsmXL7ODhIzLdYPRsVKTZOfEgkDzXqCdESqjq33RBPzv99NPlPl555VWflVeeJlNZRplY5skHNhWZ3X5w337VdwFROPljI/gCKMyubQe9mWIGN8eFUd3iQo8cPqIFBIgJuhTpAj9jgUhH4KHNLlQM0ueeWLv4IoI790e0ZdUpz/Sghn5296XkufhbfBQ3XyEKlgrRNjA0bHfc+VjqX/dCECfkkkv/0UuUkC2ItDUPjyjegy2weqwHWDhVPRYo6GROpXZBBixE4ApE1ELIcj7eFGtB4DU+MaZshw3Ha7B6vI4xqd3Hj5fMNRaD58f7RyoWMK2eX3m5pmxj6mlYIZClfqLIvTwj9PGV3X9Q8ByQeBworFkmETKGhgeEFH70b/5ve+WVPyjOwRKQdqq6+aV7b1JExFA+ThW+Avwa0uNbb71V0nalGAIRAL8DnYoNwEVxkpwckU8ivFm9BynOosULhVcP9PVrE4AVYKIo1/Ilc79okS4KdM3fF1yd0qVTukh9hEgBJKX5N/hsGh85daSU5RU523TLXV7ISHAm17N8+ee1gQjIdJLLoHwPWVNrs9OnoECNg3Hn9XnBrxNil8yyePXFokypQ8KO1g0yb0aTKpzsSNArOLYwYVXM8ZNoErJsY4oTsKq4Ew1KTPIuXFdYPtfZcUAM9yRO/8iwm+k0hgW1UVf28InaYY3405FIpnJ6O/fChfM1WetY93H78Ic/JGyGQ0j8w3VnvnzfzZpJozr05KTKosLAJ6EF9WsRPQqusDmdXjsHBZLPVOHAmzD49wknnKBAqm+AzeCFUzYF74OvB3fHPNU3NmjHHj58SJuFgUR8fmDtRNzk69wQn8vCn3rqyVrY3/3mt7ppzLI49pr5WrCtux71lqfU5oiPX778ApueZpqFyarMaW93WlW6J6BZTljQjtU7l+bJKU1i/HdquCC1YvHJrUVSUarkEjBu9oFq6eLxfJ8TqxSO/rnBQVGnAaWcdeMkFlkVJlkeOpKmZHvAhyHTJkqoJZ/rC+uEjEA0eU3w6LznYcqytLEVCiLWiOGUMd1zjHANelbm649tK2LKtFBJBgSTD/qEmYcASSBDdMzDBDtXVwupwZDj95wW0gsRKnI523dgv33gAx+wg0otZtIJV7V2UQNep+ieIcOkbYqUY+eip+NdIJHiUUNXIwUnPJWBMeH1TU1Ka7bufMS5ZIlszLVecMFnLFdZptFkkkPNuKIXlTjvGBrzGnU265y3JIyAb4+/q+w5ewxZDERQT2G9FpJoHXEjVdVE+vBytNKzEa9A8miF5kFrS6eeXFs+e9QXvKWlKU3HTouMRKoCYub8EARSLPLSclTrWFzAL1Gp4RFMOL2d95Vu0ZQHkVFj8EOTdSIGIAzUIC5q6dIThfkeO9ZtrW2tCqzA6WUVYp5qIuydcMJJtm/vXsGMXr50rRwujJtvbW6Rn2GYMKeEoGg2jEjMgCUQSlbFn34CeWjE54HbRx09KmMsWrQIEfw1NzfZhk33KkZJDWtWna+0Ky+/yArTY3bayafZ7t27dQ3KsS2NRkuEC31+0ujFtQB98llt7e22f98+neQ4XeIMJhPPQgCB4sJefWW38nEYRF4hdE49G5WF4P34s7Ozs4QlsKHkgoRquuVUrj86at3dXcIgnBQCv69OmxP8JBRLmNHHsw7Xi/VlMxIL0a0r2HZkLE3ldqSRz+E6M4/fs0GmvhJcuhzpLm+KBIXjwR/rOip8ndmsPCA8F5RnLrK3p09+n5vid1h4/mRXcZMEJVJpSpuKG+Xhc+EgVSBp+HdV2sYci4cRo9NS7Qxebgy3EOlUwKaoSjj6VWZz5nTY6ut3ajChu+FpKUlcdvH5lqs0Wzhvod4Hl8P/pHf4dnw+zJuu7m49JK7t8KFDRrDLn+oM8qPq6Bh074YGReKwd3SKUtqUKy8T0tjS1KDnxGZQYWaqIFOvAk4isi5e7OVhfs5zBDDzlBCh5xG5ymgSZfGpYbiuDfGFN65geTvnzdV1URmlkMbJ5/V8Vv+gB4gEyzzv/v5eXZMX0fos8/hd16uLmh1K/k6q45Qd998hPBQSH1zsgUOH9YFwvoQNDw9qIXmo3CSRrgMLznFTE0SxqEieDwU7P+2005ReschRueJ3Gpsa9CAYMBiVpYghlPfWeQziIIr3qhFNf/FL37Lu3gGN5NCEiVzOVq+63MYV2HlxRtBdkl/DuolnNz5uy04+WYEsmwMkrSTHopGiruilzCXBrYoLkmvUYWDTV5QLJm2sdx4iETZgEQ9atXTIGslP63SDDPb36Rr4t/x91nsTCaSPH+9RysnP+CKdw18oOG1qVpoLMQX2sFrNAvXLlidhSA9EuTbdV1LRBK+ZN3++Zb5453qNJglcmoALKBUT3N8/oMUMhg5+ROVWsWkdcePGYZLyxckFatzz+htJF29cpr2hsUkLD6QIGkdEzOsw4SwqlTEu3OFFpx+B2Olk5fOCH3kdOW0ENjz8qPVjcVj4o909CmYwr6SUVy+/wIY0r86HJQDv8loRQFP/GVbjlFNOsV/+8pfaLIEQirac0sj4XnDxFBWnDhkwdbFsUutXZwdwdFdpkUOdCnUQUctQDUsR/rGuY7oHClq8jnEr/Ly7p8eWLVuqg6EYJCFydQlt1ABFla3x/04Jw1KiJ3Dg4EEVYYjRgqcYAR0HD26j+PWP3HZdkXIlUXx0XvDQBgcGBXzgD+YBeowSJdYpNaqpd9UMomi1W/X3yULIVShSLZeZyedrZaZggAqwSDNiRsZGZbpY6JNOOslee+01ZQQUQyicvP766+n389ooLHy4iKAzcVNBGmHzPfH179qbbx0QCdPVovK2/LKzrTA2ac0tDTrZCxYutD1vvKGS6FuJ78/G5CF55uINCxFb8D3BrhMTdvKyZfby7t0lBg3Xz7VF0AYjh40xt7ND18/p1eZJaKHLrngJl3QVi7d37z4vswJIqWbP73gAzPOL6hqDk72+79mAtHlF1/LFfdfpp9vLL79sdfUNSuUIltn9vCYsYxwULI827m03XV6UGTSmOfbLj0SPHHktfie6QgFYSLWYncb38IEnnniiHT54wJYuPUk3jAkiAkdJGk1WPmTu/Hm6gFdf+YNuCBkx0g0elDhwSVQAHxQRaNCTeFj8bgR4InqmICjydn722JPP2t69B0XChEgBVezq5edq4Wtq/DMwr4J5wctpDKUMevRoKSJHn0YpHOzXRMNS/AOBIaGSLBTXwCmlhkA0r5gEhJD4ZWjAq4h5ytfHpQg2o28LXa22VE2TC1Cw6ILIuFYWnqZLDpqKZJmM+A5Y2qVLl1lbW7v9fvfLugZa0kBbeR8KbFgv6OgLFsy3ffv26nPASThYUeDRCFa1UG25poheLaeeKD4wXo0T08NCCWtMgYMP55vWCBE1WKZmymmEjxgSkPdZsyBi4qGlliWoSywE9fz6hnpZADB3AidGjfUPDBr1gNjpgfJhbQQBq03awRlAkGh0ZDHxo2WZCvvmd79vv3zxZXHKYdYCb1512XmWLfrkCLmmRElSPSHx491v+8PgRPGemHwCOSzNbJ8vcIh2KLV5eZ4PM1fl5rExzXg7uH+fglI2GP/GXLNp2GQqG6fBSNGHCLuI9q7ow2NDAYodOHjImpuaSvGGqF+ogNBJm2TbyPe5D96bTIwdxqYjHti/392nGFKDrunPa5llK32ie29dUSSvFfm+ucWOHT0s8QB2fwj1xWkTzxwevSpzMzIbUIx54+a2ZlGCqem3i5yRZqAxpntoUGkh/vTAoYMGpRvMnx3Z1wfu7L43SrpRP2YjCeYcn3SZlcRa5XNYiGE06spy9h8vvmTf/+G/C/yAZ1dbU2Vnf+aTlq9w5kyAUUDLasdGIjU1kODmRPzUTLnUHpZ8uNQvEnE0zCaY++EjR5KlchYwGQInv6ba4wi+x/1Qv4+NvGjRQuH/PEOuHatIDYMNzgKxgaLMirVgERU/JJYubOawklw7B4vf4X6Ih/hZBIsE0Pwu38NKidUEIol0HPf44PbVAnCii4P55OTumOkaATW0D3t0yf+cAhC81994w1E3RBCmXU6EDhnBqML3qyxfjVBCmTU1NSp9ES2bnH98rCRH4qVCJk95vRlfxHuRu3reXukl09QCxabDrImGVVll+/fvE3y7+4299vgTT0u8IauFr7ZLzv+MlaXxKVTBcC/CABI/X5Tkujo7dOigTjlwJ1aOzIbXhK4di0MPH0GbyItJ5NDr626psHJsRip8AEsLFiy03/zmRS3k29/+dqV6eu8JRBXrFZSxIKR2xC08B6hgArTGx/VZvAfvSdPo2962xPa8tTfFOs5o4pl4EDolCBpLRPEMXOOll36n5xcnPdwGyqWsRWbbugvVUEEKhQlBQlMPRHnhuI1PTAlp4jXC4EGOxD33Sc+8uQr7CdQJoqAujLZdSYVOKpI8cuSwAsXDR48IyGCnc4qJKagtc8qxKjRa8jvisA8Oq+yI9RBF+m1L7K29e62hrk6Vw9bmNqVik9Nltv1OKnSwSgtWV1NtV1z0Wf6hoBKzPFtiFPOIxUEMghNI8Id5F0rZ1CQSBEN8hQam6pznw4OJPu5ZTrOwWAAABvFJREFUTGDvIHROBfCYJEqgRNtsXII6CkFtczpkesEh+JMvTj6nSzP3VCHEZ494Kq1NjwrYkAYl8jwbG73rlWfMurBxJLyUAB1laalbCYvgKGWSgU+/l9l+/cVFpLkwt21trfIvqnc3NGiXAtzQphMa7ZxoatZAlbBOojLEQ+ADeRBcAOkaqYMHRpzgCQWCwqKtKL5Z+G8CSJBCHoT8N0SDnm6dlob6Rj3gI4eRP81aY1uL3r/ryFH9WZUDSCmz8SmzGzdvV9Mg9KeafM4uu+AzVsyWWbWUpt2PB4YOTCuzy8ad1TDJ94Jq3tFBQ4e7lEhf6d1z7MERShaH9yBd4/5h33JdsSFU+yZAG5sUlgDKScyDBaFphA2BWed5UzvH2vL5xFguFU9KPKxaw/HeHnvnO9+pcSxYXiy1KqkpLS5RvmYri6eFn03OEPSNjxdAAfOSC4S7pTbfKevp7VGKBuEShA5fGcIIAV2qNJoeaHdXl0622q5BqdTsT8BHKbU+FS/qrLe/z04++WQtPr/PotTVNSifR6eGWvKRw4fTA3YtWKLd4eFxa2pDdRN/6Pg7o8zkGianbMfOB2xkytUr3vOed9mH/sf7LFfmvWlsnkgh2XD8OzIIrAlLywOONDFSOR4498TrMZEshuoMtEez4JWV+v67z3iHDg3AixdVvPERq4e76pw7T344MqTFixfJXfG7x4/3yvJkyp2AEvgIm4nMig5dxz8G9WwCKY0iFu3nsjKTE3JP3O873vEOcfkWzsciHJAb4Xq4LjZV5s7NVxX5UHwPPogTTQ15/779DhXWNyilU5ExhgmlZgF2rwgEaUQJf8eEE8k6ScE7cpyPRp8d+Wmda8tHg37C9slJA1o8/YwzlGcTmLS3z9HD7ek5btlsTvPtcQ9DQyPCEQBlvI5g1j80Zt954Yc2p6PFFi5ot5amZsunFqpAwBSApdZh3pdNRZFHRNNUYAnXFVg69+DFEidYsrD4V96Lf3Pdbz91qcz1q6++6n15GhA8LkugBpMCJW+v2EEqpTNYm3loWEr7YskyRSs9D16HYASvI4/n8/k8ov5onuBzvf89uIbetctXXC8CDX64YA6TXeS9d45OGrUhJ1YoJowHQu7HLzQ1tSQz5PNWPJhw3pZy/ELBWaTqb3Mcm9ewu/g5fx8ZGnS2SL5G3ZpUjCIHp3BAIAN4I1p1olmJk1dWJloWppj3amlpSxOovd9eqhaa+Ybahte6OXHeIQOciYS3B5R8EcCSe3tFi8qYVx65F+IINgHXHac+ImbftB4xhzvq7JxnR48csSVvW2y/+MUvbPHCBXpf5upQZqbRI049+Ln4c5U5mzOnU00msHZEBqFRNV+tE8n6+Wn2AktM447NiushnuF68f1oBcxUL735MrKgzg5Suv26bz4jJGe4Rlk6miZZdGrF+DOUKKKYQD66YP5CmXmfHu2Nj/gYL0WaokgCQ1XUph0z5mHGqWEx0cKXJhEQYxrnIXp2InZwgbyO3yO9w6wRaFEDj5vmmubNW6A5LgRAMHz5OYvOaaUbd+68ufbS715S12N9nevToLXHfYHaqfxb6uwdV0ApBm0qnvCQhN+ndIx74Wfcc4g68vv4V1q3+KKoJe5bf58CrUWLF9jvX/q9vfvd77Gf//znej9cBfcWamCSXU2jzvH1WAbFRF1erGlqbhRtvafHadFhBaiJ4PP5fK6ntbU9PfdpweE8R3EUYCtPeqDKCef9sTqk6/xcXUNP3HdzkZSGU8cNR3QI4MIJoFIlKtE0rcXO62bXExEvmDvPiQzlTg6I4gUXyqnhRr1Jo09/Bh4gaDhNV+CU4tvhe+MigpoEygYqxfu4C6AChabulDZM6NFyoufPW2S7//BqqVWrrtaFF+hY5T0nJrwVKXJZpoY5ROqyZgI2YNGWO9jBZ6jXL6lhuTy74+xBjOT3+Z8TxLOb0+6Wq7mlMal4e4eu9/oPG2JEFLJACjHv3Bdw9euvv6YYQPFKuReX2Ozx/vxJ3ULo3OiwGik62zt0kHg9hTUsAxuUplfiJgFrYfKnJ62ttc06OjqV4jmHcdoyO2+6rAhIAbAC3iu0h2pRahkGWXPFZ4CC2pIejqDMcl8U/G5UzXhg7PJgfCiKT6adm1C78+SE0LtIMXpT+dWnS7nsGj8DSJJ4YqI6QzKMmXFhJicnaSHK+/yY9OCERasbZkhB5Eu//40eEE8rfDrXiRuJiN3h6Ua5HDD7mKnnCCSl0y69ln/zu17r9tHoqrZJ+AGk02vkyIuhvBF1dgQLuIbe4z0lxhKHQSVwMZCnbJA6SNKpjYIQh6e52Z/HokULlAIDu/K5R7uO6WBSyeTZxrWRfkd8BTfQp0zOVDsJ+v4/WJZZZ4vk0WIAAAAASUVORK5CYII=">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -326,7 +311,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1033" name="AutoShape 9" descr="data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAO4AAACzCAYAAACO/iALAAAgAElEQVR4Xrx9B7hdZbH2u8ru/fRz0kkhjRBKaNKkKCjGC4JSBEVERLkowgURFDF0RQREpLeLqBBCk4RAekhIAukV0nN62b2t/j8z31rn7ES8/733+Z9/k8Np++y91re+mXnnnXdmSXNef8Lp7e5Fe9GE4QAOgIDfDwUOZEkGJCDoC6JarcI0TehWFY7j8MeUFgVnTWmE6VhQIYOebFkmbKsKwzDQ0NDAz7MsC/Tw/u6fvpZkSJLEz4Gj0v9g2zYcW4IMFTfe+Av4/VFEY1E0NdbhlJOOQ1fBxt7eEtq7OpHJZVCsaNDLVew90IlUfT1s00IoHIJuWDhQigDBekh+P2RVhRrwIxQOIxAI8HN8PgWKokDm07XhUxVIsiQ+w8GktjiuOi6C+qZ6xEbNgG6GseCD+Vi0aBG2t2eBUBKOraOqaTB1Gy8+di9kW8M11/0cPUUdtiNhZEzG9791DqyqiY1bt+Hj9Tthpy5AJpNGqi6BUqkMNaDDNC1IjgRHTmHbrl3QjT4E5ACi4QiGN4RRV59EPBFCa3Mr0uk0FFnB4pX7kSlbKJT3IKBYsPQOSHYJFcNAUFExcdp3MdDfiaOmTESxlMX0KWPhOEVEohYCko1oMoU33liBbNGHxi9+CTvrfbhg2hh8eKCI7v4sUqYExTIxkOuB0r8XqR1zsbXhHBx53NGYEMlj1iWnwDJN7Nu/B3975wN0ZDVojg+5ni7cdPU3UMz04Y677sT4YSMgWRZUWmjLgGQDsB1ICqCoKmRZAiwH9B/9oz1A14WvigLouoP2TAH5ShmmBfzp7p/g5OOnoVAoIBwK0VblPSY59Fwd5XIZjmTRbuKtJdF7ObTDh/ai7dA+Ez/zfk6f6eeSIiMcDvP7K5IC09Yw85qHUDT8fJ0cxwb9pzgWTEnBV49twN0/vxbxYZMB00CxWISq0N7y8fnRsRm6zucFiXaWeNDep9/9V49B+wAgyzKkt2Y/6WQyOWzp7Icl+wcNl1ZOoSdIEhTYkBUZlUqFl4CMk96IDDlabsdV5x4JRRGLrCgqLFODrmmQZBmpuno+SV4MOuBDFoh/DmnQcB1bGXqeA6z8cAU2bdiK5uZGdij19Sm+MJFkE/Z2Z7Bu01Y0NA3Hph17kC5U0DOQxojhI2HoVWiaDsu2sb8UhRRuhhwIwOdX4GeDDUP1+9h4fT4VqipDVRU4tskGK7MhO1AkCRObo/j+iTGkGlIIDTsaVc2PVatWYv7772NvXxGGGoVtGqgaOizdxnOPzEK6vwO/f/Ql7OrNYlgqjrOPGIZhbY3IZ4tI5/uxZ38Z2/om8xrGolFAlmCaVciSn51OxVSwcfsm6KXdCPr8GD/2KMiOAUmy+QOOBU3TeHNqcgTxpsNgWXnA1mDpWSRiQYwd1YrO9n3Il1vQ3t2JunAMra1taEj6AElzHYSDukQMjlXFTgf4bOJR8KlBfPmweuzsyaKnZKLvQDeGNw9HKGhDzqWRmXMPIufciExJw5cOT+LSGS1oSiaxp6MTj771MYJ2FkeGu1Ep5dE6Zhq6s2U8/sRTmDxmNMjiFIlOlyxTGJktkbMkw5XF9w6d39Cm5o2tSKjqNg4M5FA2DBiGg4WzH0V9IohSqYRQMDj4N2SIWqUCTdc/13A9I6H9WPtetYZLzkPx0f7ws+E65BYkBV/+3v0oa2T4Yi+zgbNhO/jzHRfijDPOBoJxGOUKBy+Z7Ef187nRg+zCJudSY7i1BsuOxwtiroNhh0bH4P6Ovpfefv1JJ58v4uOd7TDVAL+GLCu8ib03U9w/oMhpOxYdNUzLgmNr+NrkJIZFyogn42KtHREt6bmGaUJRfUgkkgd5udoFOtRwLZN9ED/f0DTMfvVVpJKNqEslEYtFodBx0YlJDjp7s9j2WSfijS3YsrMdhiWhUKqiohniojkO9GoVXVoEmq8eaigGf9CNsn4/G7DP73MdDtiAySh85IBUivw2VFnCqKSKH59aj1R9EuERx6JcVbFyxYf44IMF2NOf5WhuGQaqugbTsDHr5h9iTHMdHnr8FazcugvHjW9GW1TCKaedgo49e0ExoD9Xxd8WWFBVen8/VCXIjpIcBjmPiiFhX2cnejvXwjIKOGnGOZBs2gAWorEwTKMCmyKF4+CzzhyUSCtkjkwyRxafIotNSf98QN+BTWhJtMA2FYQiQQQDYcDRYBsSHLsMnz+AhrNPRldrAoVCGjNGDUMoGsauzl70lGRs+7QXMnQ0+YH4wt8j9MUfoGJJuPCYkbjy9DGQLBu7u7K4YUEPDi9uw1H6CoT9QG9vHn2ZAhas2o6Ro8bCJ8lQJQmGbcCxLMgOIKl05GDjJSPwHLzY3IT8FECVkC9q6C1VUKjo7NzWLnwRsDTouuH+rRtJbRvlUpn34OdFXEZ+9J/tHGS4nhF6hhSMhNiI6MOEhEy6iAtveAqGwZtUoEmpAtkOwIcy5j9/PUYefipk1YdiNjcYSQOBkIisAO/LweD1OSGWtnZt8KX3ONRw+ZjemvO0o5eKWLvzADKmD7Lih2QZcNjKIUI9LSihGItgnA4TCvyOhiObwzh5HCAbOi9sNJ6ETl7MMGFZNgxDh2QbUANRROMJOA4ZuwJIBrmHocgqy3ywtkUeTHhdOuAP3p2PSCSCRDKBcCQElY2JsQW/1qKFq2H7gkikUti4uw+VchWG7aBUqqJa1WHLEsqVKhw1ii6jHlI4igBB5HAIql+F3+eDSh8EiSWJoy5DZFlGKKjycRBSaw368NMzkkg2tiA+9hhUKj4sW74c8+fPx/6BAuxgHJZmo6iVYRs6rr7sApxwxOFYsHgNnn11EZriCqaODHO0PebICbBMA7v3d2PJOh0FNECFClMvwbIcyKqCgBJCsVpEpH4kdu1YhkppP5pSDYjF63DFhV9Gb18/PtvdiXK5gmAohO4BBUZwNPyqCsumjUZe20E0GkCpWOHXHejajrp4HVQEoUoyTNPgcwUIIZl8/kWninG3Xo3S/t2YOmk8DEXCZ305pNM6KrqCge5u+GIJNMx9APqkmdAiPtw+82hMa9QwqmUEdnXn8KNXNiNo5zHSOoDj5U0YGMhjIJfHkpWfYvSEKQio4Iir6yZff1Wha2ox5GenLLsGYVJEk1yoTNtFQrZcRW+2DMPUeS+u+eA52CahP7DToy/IGC3bQqVc4c8SuUk3Onohmd6XIPOhhusZI6dpcBBLJIZMyzbx4uyleOqN1bAc4VzYJmxyNgZGNIbxyu8vwvBJZwOOD6V8cdBYfX6K2oBj2xzMhgzXTQ9duHxoQKu1axGFh+C09I83nnEqpTJ2dfVhX7oMS/LxG9hsHAJPB/w+vrDk4WWJFkNGWyqMeuMA0rksdn66E0FJx29uvgQWG54wStMyYelVmI6Ozv1VTJwymhfRkil3FHBI5CQyDIMWmAxXZMtbt25BYSCD+vp6hCh/USWOtF6ebNkm/v73f6Bp+CjEonFs2NODTDqPctWA6g+gVNLhyDIqlOtUHKT9bZDDcTbcSCwK2afA7yeHJENRZAHTZN4f8PtUBH0y5/h0nC0RP244I4mG5mGIjjkKhhnCwoWL8N5789CZrcAKxmEbQKlcZHh03lkn47KZZ2PvgTRu+vXT6Ow4gNOPGQ6fz0HE7+CwEcOQTmexaUcPDuTGoqrpkNUgZN7EMmQfIQoTajCJYv9OdOzbgFhYR2NzE1qTEVxw/plYt+UA1n2yw82f4tjZVYaqhGHLIYEiZAWOJMPHMM2Hgd7dGBjYiqAPCPqTcBxy7WLj0LUNBANwNBNj/u1ctE6fhnFjD0PBtNGXTqO6rwOObaA9b0DzBeG89zSGn34xtvRm8eSPv4rprT7eFzs687j6r3uR8pvQynlM8OUxrOt9+FUFz85ejCOmTEDYrwjD1UwOQbQfac1p/RlJ0abgvUZG7RPBw6fCtG30pHNIlzQOCC1N9fjHK79DtaLB5/MJjOZyL/S3lNZxoIEFmwy4ZuMLwxWG5BmLB5+9/UVPD0Wjg7CVHOH1v3oaa3emYdrE8QjHQq9jyRK+f95R+PGVZyI54ijYugWtooljd1MA+to0DE7dPCjM8Nt9/N/y3H823DnPOJWyhmyxiNU79sEORGFYFixb5Ld0IsGg8Bj0vSzRgquQLLGABOvWbViHancGC5+5FgHFgcMeX/xtuWzh+p/9Du1dFVx2yRdxxcVnwaILpci8sLyIJkVb4U1sKCBHsmnTJs6bgsEgX1QLdBHEg55pWQbefON9JJtaEAiGsPVABu37OxGNJeFICvoHcgypOrr74PMFYDWMh5JoRDAkDJciLm1wzuE5n5XYcBWZ8hUJAT9BOkIHNlKqg1vOaURTywhExhwFywxj6bKlePfdd9FdqMLwxwEDKJbz0EwT08aNxi+u+y40M4CvXPgLZPN5HD0hiZZWP+pSKUhaGU31dVj38VrsTsexZdNmtI1s4Yt64EAHHQRikRjidcPR2DgRDQkL06fGMG5MC1paGtHc3IC/vTofjhlCT08X1m/egZIdQH/GRDCsMtqhTeVXJRBMI5YiHE2hr7sLo0c1YOP6tUzYsHGoAeYi/H4fZNmGKsVx5oP3IkBOLRhAbKAHxw68i5FNCV53XcvjP19ZiONPmoGGuhhOPOdCdGUqGDlsLLLpbmzZ1YXOTAk7uotoVVU0GxvwwdJ1eG/pGkyfNgXRoI8Nlxy1iFoUBhzeD2KPkVEIo5JlkfcyWaXI6BzIoj9fheRYOOWkGXj0rh+jWCrD7w+IvUEGBQeWaaFULonXc0R6d6jhEkT3jJQ+e8fiwXQ6nkAoJN6fSCjbxDeu/QP6SiK/pSAmILcKWSrh+TuvwCmnngwn2gSjXIKpCV6Hoq2XchInQScnzon28cGG6x1DbaStNeyDI+6cFxx6wXw+j1XbPkUBIZiuN6YX9zwhQUpeG9vkjc4naBv81rlcDls3rsG5R4zAb/59JkcpQ5ax89MO3HjLg6jqfui2jnAwgCsuOR0Xff1USGoYNhm4ZUM3CbbQK5Gx+HDf3ffAMmUR9RQFyUQCDY11aGltRENDHSCVGWqt3/AJLKsevkAIn3VkUawa0C0H+zu6caBzAGogiGgsgT3daQSaDkcw1oBgLMS5G0UYiqzkrdldsPHK7HRoC8mSLTavLCNoWbhjZhPaWtsQHX0MNDOMNWvWYM7rc9CercIORkDeqGIUoVdNtDbU475brmMS77SZ98ExMrju+2fh+GmT8Lc334Bsy5wv+n0h7O1K4d0P/go4Oh8T5dm6XmGSLxCIYerkmYDUjWggjRt/+h0E/UFOXwgmd3QeYPZ007Z+PDdnCzLp/TD1XjiWAZvRggk4ClQ5iFPP/A5WLF+EaUcchfXrP4Bl98Mh1FZDhKi06UMxfP+Rp2GnGnlNRvRvw5HlZYgEAwhHVISCIa4weGzvmKMvRFHycVWh78AO9H22ktezq6sH7fv70JctYf2eHDZs3I6Jk8chFgyCAAXBWK5a8FoLR885JuVvFCdti9MYj4El8NrZn0WuojH0v/m67+HbF5yOYqnAzp1gr8cq67qGarUi0JxrIl5kpc3PP6/Jb2ujrWcojDTDIjclY9MNA1/9wf2oaH7QVmXiSZahUOrns7Ds2e+jZdJpUKQQCoUBSA45UMtlpcXL0LWqfdQa7ucZa63RikA4hBCkd9940aGDIGZu+9792J2uIhiNI18sD7JYnD9wDkjQcsg7yQx3KQoDH320HAFNx7Lnr4NlG1i6aCneeH0V8mUdVd1kOFhiRs3Ed751Fi666GsMMYjrEnmKgObLl67EiiUfApbId8jzOZaNUIDIJAXRqA/1jQVEo5R/qEjnYgj6QujOGXh35Qbsbe9DIhLD2LFjEI4nsGnbLhzIO1CSwxCIxBCOBBGJEUnlRzDgd8+JclmBMCjvo+iryjaTPcQkRmQHd3ytwTXcY1Gq+PDJ2rWYM+d1dOU0WMEoHEtCSS/BMYCgLOHxe29lVHD2hQ8iFAihpa6Ec04ehzETJuAvr7yJdRu2wLJUnHHmJZj9+n/CsEqCA6B8T6GNHMDxx50GvZKCjh7kM/tw0w8vwbhxTcTxIxJOoFQsorOrHZt3FfHsnA5kB3bBrB6AY2XhEPPMgddBou4whCPHIp85gKOmTcWqVe/BsnshgQi8Wq9v4oSTvoThF14Ju60VMSqNZbM4r/wGI61EIopwKMjGRAZsWjZGH3UBuopVRPwhdO3ezIbbN9CPnp4+VMsWduzpRE5twOqVqzBlymTEwkE4xH0QQeVufoLSTKR5ZRoi3QjJ1+xmw7LRly8hUypRpQXP/PFOHDd1NEdWMlwRcYVD0DQqRwpy8vMMl1/ZEsTUoaUgj7kleO4nppqDlYWiqeC8q38LnegZm/JziqiCT2gIGnjz6evQNvF0SE4A+VwfVMnPTt/jZWzLYkL3f2O4IuqLGO2t0aDhUk6QzuexcnsHlGCEa4CcIzA8pg1NueAQeUAHRAYlfCYwMNCPLRu34sGffAUL5y3Fkg9XYFxTBD/4xnFQ/SYK2SoyuRIMUwGR180jx+O4U06FYzkwyP4p4beAmd+6FhWNDlCCTBfCshGNRhAKKQiHA8hmswxnJRAEUeD4FZx53CQcNnY8Hn7+TRxx9LEYPXo0ksk6xJIprPxkC95atBZWKI5gJIxwJIJQJIJwNDxouGSoDJU54eJ/8PuEU5HIcCUHv7mgCU2NTYiPPQ7lagCrV63C2++8jfZ0BXYoCttwUHEMmBUTsmXixT/ciXKphPMufwTZHHEGQJiIp7AFxwxCkoKgYF8fj2Lfnq0wtDwzxQ50Jl+IufzmhZdh4/pOpMv7EAr5UBeuw+XfPBqpxggTTMSyU2R55fXVeH89UEjvAcwydG0vR3AyWhkKxk8+DwN5BY6RxfRJh2P5h+8CKMD2nIVrNFSrnDrpTGRDEQw/YwaUxpGYFtfxZX0hfD4LwUAIkbB/kBfQdQvjZnwLOUuGrRnYtGoxunYsh2YYyGULyGbK2LanH+VwK3Zu24wxY0YgFgxAdmwYZAFknLbNXEPtw2aoLwgpLxoaFtBfKCNdKDCBOeeV32FMYx0q1QqCQQ8qi/JMuUxEnyhZ/k8MVxgpQXSZ0yjVI5UcG3MXr8Ksp5eCDNCrnBA/Qsjm3uvPw8wvTUW8ZSpMXYamFSDZxKGI8io9n2yJUqH/qeF6rPY/Ge4/3vxPhyhqgsvFQgGfbN6BPtvHxIa3aH7Fz19zHkJ5oELlIsG6eqUf2ZGxZuVHMHUDl55zLK6//EuM9Z1KN6qVKtKZNDID/TCrZfhVGUEiqIJRjD3meE726QA7duzGe6+/jkJRh6P4YYrsBrFoDMlEGLG6FJcT6PndPR0wDBnwJ5Cqi0GzVVSUKKKJBLPb4Vic2dLO3jR+9/SbgD8GNUL5bQzhWAThcMhllVXOuchz0jlRfsvVJoYmJp9zQJVw/8wWNDQ0InbYsdCrYaxavQJz352HfdkcDH8CtmGjajswqzpM28LLv/8115Kv+dmz2LSryMgkEkkg6Bfwj6KN6iM0YbIoISL72UkRdFdhcU5HHrp3YACSkub6X110AlQqwTJBSLyAhWRdmNnskjQM7fu3wC8XUCz0wrAKgK2zcGD4hLNRzNporIsjEVexaeMKhEMqKtVuEKwUD4KpKUyfei62bfsQM0b146YbLkYIKnxKnllbZuOJA3DJvELFwLgTr0C2VOVIt/wfrzGZVs7mkS1W0NWZRY8RQFaz0NXVh/EjmxFWVdiwYGhVvrYE+wXxKQzGE+uw3brf0/OqDtCbLqJUIi2BhGX/eAqRoALbMvm6kQPgNbFtlIqFQeKJN6kLj5l7oW9Z3OOWgtiwDgaq9BpUzQAhH0eBQSjxlqexp6sA2ySRzJABUgBe/vSPMGriZCjRNujEJrvkFeXe9CAcRdeb7clNTQQpO0QO1gCfwYMZKgV5PyI7ETm39ObsFxyCFSRWoGL+nvZubOvsgy2LNyXoKFFdlxhPiS4veUg/wxOCuLTZaAMR2bBl4yZolSoOqwvhtSdvhc8JsKF7LBoLZajUxAdNsMHi8o1eLsImn0BMo15BVTNQqlSYVKGLwlAl24mBgQHEQn7s7yshFG+CpgbQnzagBMjRCOaRVCrJVB0Un8rOiC7nDb9+FAgm4YvEEXYNl45fCC9UdiSKsF4mSjzhCUt7HKrrAg98vQ0tra2IjTkWphHC0qULMX/+BziQLUL3JWCbNsqmBVMTkeT5+38JvZLFc68sxe+feBeRSJyFDcKLEyynPFeFY5oIKn6komHOa5nIcCReg3JFY9hnoxO6pqOx8XD4fZQH+/nYy2XaNhZylSL8yeEY2SzhxceuRkXTUSxXUK7o+GxnN+56aCkG0n2ApaM+kYJjlZmIAqqQ5Cp8ATp1A4rUBFluxuYt7+DbX6jD5ecfjkgsCVkRiEt4NPcYAZR1C2OPvwIV00KxVMLcv7+AysBeFHI5FEoauruzqATq0ZMrsUOvT0QQpCgrO7BIrOJCR495ZUEEGZXjCHRHXArVYh0gW60inaf10LnKsXzuU7BM4gmEIkkwWsII8/ksfy/qwHSeLpHkGS7tWfd9DjZZfia/XiQcgUOGa0msirrkhkexr6cAIgYIGXqQmljy95+5EiMmnQpHjaCSyUNxlYB0DuyU4HD9VhyPeLBRDuLVQYL/0MNhJOgFULZHlx2X5rz6rENJM21yqn3mixUsWbcZlhzgheMnkkzQ3VSkcmEP5zgI+Ag2CW9JBrLr08/Q19OLsKNh5euPspqEuTPXy8jMwokDIWN0qKxNTsiWUJUcKJTbUCQmL6dbkH0+UViXJQSkAG6+6UZU8n24+LqfoOyQ2siBZDgwbR2VquYSHvQ3VI8G18wIkl13+28hh+rhT9QzxR8Mhxl+E5PKG4QgJW1OVomJTcPHLAlYpCoSfvf1VrS0CXLKskJYsngB3ps/HwcyZZihOi4BlHQTJknaHAe/vvZyjGprwPtLV2Pb7j5YpgPTcGCYFtIDWVTKOspGGZV8EX1d/ahLtXA9WcBHKtTTcx3ouoJYjMwzj0J+AKbhhyrH4Q/4och+2I4BWY1AbRiLpoiMvz75HT7eQECFLSnY9lka37thDnp79wOWiZCa4DTAz+UuujwCTdF7F/ImLFTRn/kYt1w0Aqee0IAEIRN/lEk7TmBk4jkEE7+/ewDTz7oWhaoBzaji5T/9AXapm6FqNl9BoWgiMmoSPtm8BZFgCFFFRpA2L103xxICCTcKUTpWy6p6m5UdmSQhU65iIEdSR4ed96I3/4iqriMYoDx0yHDpNSnieqUhQlK8prT3aiIuMc+f9/AMNxqNCqEk1YR1BZfd+Ai6shoss8yyXK+Oe1hLEK88eDlaJ30Ztiyjmi1wGsOkrquWMmxxrrXB/X9iuJ6he8fL8Pmtvz7mFHUHFc1EqVLm+tf6rbvQm69A9gVJzsIqHM5xVSFpZBgj0cUX5RQhxwJKxRK2bNkCx6jg2m+cjqu/PZNPwjPcIY9BjsuVmx2iYZZJ10nqIVa2uAbEb+hg9it/weN/fh533XcHjNgw2FSy4ryBlFyibkwPikZ0POSMtGoVT7/4KjbsLiLUkEQ0HkcoHkUoFB6MuMIjk6xTASlj6WvWzhJ5IQE+MtyZrWhqbER8wrHQ9QhWLF+MeXPfxd68ATuQYqOoUv1OE6TI+eecgW+ccQIKpSzLIelBx0JsOCl9mEF164tk6PRG9Ds6hXSuhFKxikymhP4BjevDp37xSPiUMhzbh3S6jIFsDh3tnejv70P7gQFkzDZEI3EMawghlYrA55PR2tKCiqni/cW96O7fCccwkAin4AuG4VcDzHIqfhlUDqRlLJd02DCRL27AQz8cj+mHUXpBjs67znSph67JrgM5TD/vGlimjWK+hNee+T0qxQFUqhbGTjsOXekqetJpLFm0GI119fCTcyZqjYVvQ/VMj3xhYyAipiYaUpAgdplUcgPFCkzHxsjmFN565bfQqkRaimqHZ+gkIS2XCoKpGvy5iHOsU2YbJ2XfwfmmZxQE+Wn/hUOkUVZgwkBH1wB+ePdsRnwCFVD1wWTE9Kurzsa3LzkewcYj4FRMvsYsgXRhMr2up0/mczvIWwwRg14Er/31obXbg3732aLHnb29Rezut3njFasV7GvvwNbdnZB8IRH1fKqraiHjpbrVkKqKYJuAKiKSbt68GVqpiIRcxtI5f+Z8YjDiuh5ILKJQYnkP78AlRXj0SqWKUHCoAE7L/OnmDdj+2R441QxajjyDYTY7VFcaR8ZApI4HgzivIK1y1wDuefSvCDc0ItXUiGA0zLU/IXEUOS0bK0dfCSrLBQnKCKilysAD5zWjrbUZ0XFHo1oNY/VHy/DevHnYla5CitTD0nQm2ei4CU20pSK49Yff4U0fDoawa+dOTJgwwd1gYv2IlffIBzoILoPQktimEMEwkqE6pMzFe8OgRg+dy0UiehuiZpnpQX9/Gc+9uQ29OQOmYXGEN9xIWjUIHSXQ17MTjlNAkIxXjUCrUp5HJQoiIKmgI0NS/SiV9uDF20/D+NFJ2E4RPjkoUiZeZ8GU0rGtWLMbX/nBr/jY8tk83n71JYwdfxiUUAP2dvShK92DXN8AlixchGQiCR81oxCooLV2RRdebuvVT739MFjjddFPX7aM/nyJhUGXnv8V3HzdRdCqGsKhgGhIcAk24lM0rcycRa3hivRMyA5rm14OsiMBqhmxEdcgCmoGlq3Zitsee4+5Gk4XmVC2+PfL/3Ijho2bBCXQBD2X5+OgaxIIR8RLu6UkjiT/pE8eMtxDj8OzGc5na0p23jlJBz563jF1DX35Cj7emUah6iCdyWL+ivUccYPRCBM0JLimjU1Cf853yB+RMscnch6XHUdXVxf6OjqhOCbef+5OJBNDxudBB2G4Q5GYWEQG0czqEsRwFVI1EZeEGUYpi83bd2Dz8vcx6ezLYHXUJFMAACAASURBVPBJUQRwSTJaJK/7ggorlMsYJgbyBfzi3mcRbx2OaF2Kz4maC7zcypPZ0XmyGGDw/BQu0RCsu/9rTRg9ciRCY46EpoU54r4/fz72EHwKJOAYJkxHZpaXan7JgIQ/zroVlmPAJ5G4YUhg4F0kigCs2GLn4fHzDovumRxwyJS5rUUoXQm9sEMhdyK6ZugfEWoWlW4klXQg/HeGabNm2zaqLM4nKSqRYNVSFoZEsLiC9EAOezu6kM0UOOqWKsQtqKhWC/jWKXG8P+99zDh6HGZMG80IhYT8JjU60DEDWPnxAZx79W0swunuzaC/vweFqo5cOodcMY2O9g6EQ1H85aWX0NjQCNU2IdN6knF45Tc6drd6QYdeK4Qg02NVFEHlos51XEcGXnriARw5vomjG9dwXcUUfSaexrJ0l032IrFbu/1vGq7fJ8qEkC2YtoSb73oKyzb3uVSpyzzDZqJxyTM/RPO00yHbPpQyGVfCiaGI6xmue9H/VcT9rwyXt8AhjQdS18fPObRYtOGrpo+VL5v3prFu2y7s39cH+AMIx2MsESTjJT0sRWF6iIglDI2pcdvi1/ls+6dQZRU/vexMXPJ1OinKlwnGDhmrp0cm+BFPJoSHYwvyNjA1wAgWTexFyqJlzJ07B5n2Tkw45Rw4VhimQmSGDcu9eBRlCS6JPFo0O1DB/me/fBRGOIamEcMQikcQcoUMg4ZDqQBLHsWmFBFRgiXb3NJ298xWjB09AuEx01GtBLB6xVLMmzcXOzMGrHAKEhFTJCYheK5pXPp56r5bQfXH715/G0cs4glCQT87wNbWZoxoSDDhNXrkKIwZ2YqoP8A1cDIM3ZLhc0j2Jwg6Ph9Sj7kX0HbIcAf7MYauO62fJNaktsBPZQvO+zjrcL04i23JH4jfkbabriWhDSLk6BpRC55qmUyO5fJZVKv9qGplDPQPoFx2cNzZX2NisrtvAPs7u1Es6yiVirh71p24+qrvQfUF8ecn/oTmVAphejOviUWRmARkVEHOyJXUkiKJzlE0CIhcmn6fq5jozeYhOwoWvfkEEhH6W2ouoDyf64lMDlCLH8Nk9yJSXsuojzMqcf619dta4sczEHLqvC9ISGRZOOfKXyNTFRGU9xqhMBs48eiRePRX30DzmJPZWZZzOf47Nno3paS9eBCa+Dz6mI/YhfPu9R00VBdJ/JPh9qx9zuFNQR+mwdEiW5Tw8ltLMHflTij+CKYeMRWf7t7JjCiRIvFEwu388fpYRZMAlQmohW/7th1wDBtNEQPzXvoDQyPR4TDkOTyIS9G2kM8jmUzyoVMOzZSW46CQLyIeF0JvWi5SAX3w/tuIROphGjpCreNgugw7HT/lJ/T+XnGcFo3E9ER0zfr9k+gqSmgaORzxVJKZcc9ZeGQURVeVWC3PcCUZlmTB7zi4a2YLRo9oRZSaDMoBrFy2CMuWLsG2vhLscB1V/hmmizyWmiscPP+72/nrS39yp7thCaEIpRZvGHdN6Ou2hA8NkoWpk4dh1cZdWLlhL8PJUDiCYCiISCSKRDSIQCCIRDyBpsYYhg1r4xbG1sYGpJJ13FssSSoz5HTuEtUy3dqhR76xQTuUR4quE2om4fXmHlEPFdB5O1AcarhQBGHIcJqgtIyqVmFij6A2VBO2IWNfVxe6+tP4aNUneO312bANDTffdBP6+3vx1OOPY1hTI/ykTnG9DfEGQn0lHlTjpPIdOW4my0g1xShMkIx9uQryFdGK+MmilyGZFShqDVJhMYWNfD7nGq0LlV3iiq6HMLyDO4J4b7lr5BkHrTedK4lhDEvGGd+dhXKV0Jd4DVuiNhsVd/zwbFx20ZkIN4yFSalShbgCWxBmruGSymwI9oqU8vOgb609H8QJHWLQ3jlI3Wufc1jVQUl9tYJqoYRyWYM/FMK2/Xk89dpyDBQM9pWkJgmwiCHMOk7aeNSWJgQMChe96U07O3tQGMjCp1pY8Oz9iEXpovs5EngH5RkuEyQ2XRyDI5JFulmfn3Nq5ni9xaJo4/jQ3bkX/fkydm9ajZYjzxyMtMK43UK3y1YK2EzG6+D1eQuxYOVOJFuaUNfUyAV20pF6UkfBIjtsuF7E5RYz2YbPtnDXzFa0NjcgNeE4VCp+LF0wHx9/vAbb+8qoqFGGoQTNqfZaJYG76eCZ+3/O8r6LfnzbIISSub9TkGEE8/lC2DaSYRWtsoEjp47Avo5+zFmynZ0T9YN6qICCKUUkyqGI9PM0s9Tw7UUpLyrQavgUkatFImE0NqQYriYScSSjIaTqUtxumYzFEIvFOHWIxeO8JtTU4VeE9JMdEkdwj+Bh+o6dA8H1bDqNluYWbPp0N554+jms3bAJDl1Ho4o7br8N27ZswquvvIyWBNXgqZ9Y1GoDPoEk+HjdmjStH7XwCQZYlCJFLyzQNZBHUTOYEP1o/vOQjLLYI16KQa2mBkX7koAKnsqo1nBrIm4tS1RruLSOdP7CoE109ORx/o1PcJ3eg/EWCBWpWP7cjzFuygxYviiMcoEbTTyZI+nl6UFk72AmSzmuLerTtQ/vfL2f/bcMd/+KPxEi4YdR1bFly3a8N28Bxo87DKPHjMawMRPw47teQqYE7vUkqSCdGBluMBxhY5aIbeacC5xzkLpp3/79fMA/Ou9YXHX5RXxBFDrhWqxu2kxsMJqxLCa+iBn2hyJQqNRUU+fyOEASDGzctAlrly3BUedezJMRmMgRtQpeOIKqBJmZpLIZ2GAgncGvH/pPxBobkWhqYQEGl7gIiioSZJUWlcK38PIcDchIZBM+W8JdRE61tSA1fgZKZRnL3p+LVavXYvuABiuU4IkOTAgZhhg4YFl4bNYtUEwDt9z3Z/RkM5AUHxziCwjNUsC1BFtvwIRP0jCtPogjp4xGb7aC5978EJIpwxcQm5PzYArBlN9S1CASjjeX2OS80VwJn5fzeaQdfab+Vc6YiQ+QHS7JGIZGrS01yjgfrx0Zu991xuxguEtM9GgHaQiBP4D6ZB3O+9oX8bVzzuXOrY/WbMQtd97HnUiU85KTvv7a72HHp9vw1uzZaEs1MO/Bx2I7/Pqe06RrRpvZg5W1ZKYjK9AtG129GU47Rgxvxtt/+Q0qJSAW9rP80/V+zN6S4bLc09Wcc7p1SOViMBi4TfC1RkTOgpvyGShLeOHV9/Gn11cy289+jI6VCSwdq1/5ORomnspcTyWbHyTwWPOgqLy3KXhw6Yd18Ac3FXhOdojfGGLHBc8zdGR8LWt+IA1seM5hNlbXUcxX8MxTL6OxoRnDRo/EmLZhqGuIY9GmDtz3xDuQFIJGAi4TbCZZoUyazlCAWUm6EMzYOQ727t3LTm101MHsJ+8REccRF0hAWfrWRrlY4uhBzoCen8lkEIklEIxEWEzheUPKYfkhAYvnz0NfxwFMOfVcFCkMeVDfERCRPjzDJa9Ji05tgNf/8hFE6pvQMKwN4UgMikr5uegM8vJIoVl2F4zgNxmu5eCu81oxavQIxMYdDa2iYvG8d/HhilXY3l+BE61zZXyUU5vCcG0Hs356FUa3NOOPL8/BstWrYMsqVEtlgo9guUGmJ6vQTAthWcdRDXFMmDiCHeRDz/+Dtdgh0vZSzsk1bTFKiNIL2XZQJa0vORzSWrmdVmy07ugfzyD4Z27nDDszlrDSMAoS0IhrQamDQQKYwcYSV3BB6YtM4htBlDGh5xKTV1xyAa64+Js8fGDhh6sx68E/uq14JGJx8Iv/uBaLFy7C/LlzUReOIEC6c76MDqgRj5w+oQeueXKaReIGKsWJJhbarDROSTMsdPWmWc134vHT8dSD16NUMhBx94zYFg5LTNlQXMP1Jmx4hisMxW2i9wQbNVZL78f1cR5mQCN1HPz0zpexbEs7p5GDdWbLxtknjsHDv/wWkqNPZMKwSow3iXWIq3GlkGS4hMC8CHuIQGvwnQ8yyEMY5IOjMPE2LvLJbX2BySnabO+8+Q5UuQ51qTo0NNbDFwpg82cHcP8zc1G1FDhU5yRvTOof9kwRhBMxzsHIyOgARA0W6O7u5oVsifrw9K+u5KjI9UNipSUgGo3xpIlqucJCDhLMMyFB+YbqQyQaRyQWH4zQg4YLB8uWLMa6lcsx4+RTobSOdw2XAyRffJ6+4ZJUJPRnHbRZxX/85gk4RFANH44wvb9LFFHvKpdEXEb7nwzXBu76agtGjhmBxPhjoFf9WPju21i9ai229pdhBOJQJUIPYjIIQWXdsPGTb38dMyaPRyZbQUNTM9K9adh5TdSMKSKo1DoWgOyXIUdCiPooT7aglUrY2UNCBgtVU6AHypUo18vl85xH9/TleLJEe0+/iMLcpO2q0hiSDbW4MZrynCVbjnAAzE37RF02m80w++1FQYLBXjeKKgvikDckOW8yLknCz677ASaMaMPEw8finQUf4uGnX4SP5bEW/LKD6665DCsWLMHyZUsQ9QX4fD1HEXAFCpSymIYQt3qkIh2PcPBMx6GiG+jtz3EU+/bFM3HzNTNR1g0WdXgEHO2bcqkoXqPGcAUUo2d5wp/Pr9+y8R9quKaG83/0IPZnqCwn1pgexN4/8ZuLcNYpM6A2jGGZq1UlfbkhpJL0jrKCSrksGHhP5lgb2mu+/l8Zbn778w7pL++5/wW8/e4KDBsxAsNHDceo4cNxoLMf+3uK2NbeCVtW+KIodAFcrSoVmSPxGM9v8gfDorOGk3qHHUFPdzeSQQkfPHsPbMliVRItABmKbFqsaiKpXDAYQi6bY8KDapBkzOTZQ3XxQXKKYBLlN8Qi9nbux89vuRNnnDAV4864EIZFr0ksJHlKmwk2ryzkko28TE+/8Ddsas+jeVgbQvEEvx9BP4uQgNuT662ngDZMSPLgr/vPH4GRo4YhMeEYWEYY8956Ax+vXoGt3QbMcCM3mlN5SjZp7EwVti5h5qnH4vvnX4AVb6yAUwoCVZlzZtpcZCB0Tixo55IHnR8RQRThCOoR/Ddg+2zOP4WWmPo7FQSDVJ5z4A8HEIyFEUiFsD+Txe33PIS8prNEj6SlXFvnHI+rbKJBnZwas/Ui33JkEdm8/lJO9bnrRaAdzxnTurBTptKd4/Da3XHzDTj6iIkMHd+evwRP/OVVhtMUxJsSUXz11OlY+/HH2LB2PYJcTpShGzpHVR/X60UE95AaiVeYnPTQFaVQZABVA725PA8l/OOsn+L0Lxwp8uRAYIgDsSwUC0U3PxZSVeq59R4eKTXYDcQ0sxuBuaVU5J5iOJxIOyi9+MJl93KrKOfhruHSMS5+7mqMnzIDUrAeWqHE50TP4sDE7fsSpx2i1Hew0MJzEt7hfR6z/S9sfPDHUvXT55y5763Ev9/2AoupKUeh1q2pkw9HS0s90vkC1mzeD43ADeWDPClClDaUQICVSKQLDoQifNG8aXZ0pvv374Nk6Vjy1z8ipGgiMfdOQhKb1svHPAhAhMoQC1fjHW1R5qHSzorly3Hdzb/FT751Oo6d+R2Y/DomLEkIKMhw6XUJ/hNbyR0dkoRVn2zCy2+vQF1bC5INjbzIPJrHJ5RankzNg3MEKemYKZreM3MYWtqa0DjpOJhGBAvmvoOVHy7Fp/02KoEUyztpjpJtUS23jEkjm3HzpZdh3RvbAY2YclETpjYh0oYzqefIfHykt5Vk6h7REQ7T0DOFCTUOiyYpcUSDB8kYaepAMhV1yxIWSw2jagRGtIopZxyFWY8/g4+27WSBfG03CoEKWj/elK7x0eant6G1EnBSEEJ8XWzRTMAbj8tFYs8QLPSuz32/+jnK2T5MnTIZr89diL+/+wEjCVru8SNacfnXT8Pzz7yET7dtd6cdSowcOGq5wgpKkYiNp23BbLw0NErHF6TyGJAt0IA9mthoYuHrT6AhKdrtvPRGnJOFQp5KQaJ0WGu43kA4z0AEXBaKO36+a7i0CNFIlH9GFQq6Zid88ze8LqTY8gw97lex5C8/Qtv40+D4fKikxXyp2mkX5JQ5fXHX1tM+1BqpZ7i15NihxNW/MmBp2Su3OFde9yDyGimEZCYe2lobcMrRk3iwmq364QvH8dr7a9BbKHGbmOclZV+Ap0n4AoIkYMKHciDyzI6Dgf5+lkGed8LhuO36K+AjscQgoyY2iPA+okDueSLvYD3HK57nMXE22tv34BvfvAbTx7Xhmlt+BZ17dkm44P6lI+qAJOwW8Fv0QqYzRcx69BWE6+rRNLyNaXuewkc1atfzC9gp4JXQVVPwMznitrQ2oXHKcTC1MFYuXYxFC+ZhR7+Dii/J4nMGfJaEEfUR3Pbti/HRq7tgFkUOGQj6xEhP+nAlo0Q8eudNAwQo76Q6L11sPmYaWkDjarlPlyZOAtEYjZMFR1yCspSn+ijXI8Y1KWPy2VPx7VvvwYBG8sCh+UbE6guyina5KMsI4cOQ4MTLY4XAwpW2shELldbQtRLr/PA9v0ZDjByNjRf+/hYWrFrLLXqaZmHG1HE4dnwTZv99Dtr3HWBDpbDvGS5BbZYzqpRiiYkSwjG7cJRQCKES20auUEKupENyNHyy6BVItu6W1Ya2NeWTNCBOMLT/O8Ol4yFy1TPcVWs34fr732HeghpYvP35hSOH47l7L0F8xKlcS9bpfWlAn6dFIHmrSeo1IumGorln+IP72/3if2W4k+plJ1bXgC9+4Rg4RgnTp00k14yq6SBXtWlOAwb6s+guaDyKdOeefWxwXLLx+ZmcolojDdCicgIzj/4Q1wdtW0NfewciUgVvPv8gE0FM8HMvgVvXPUQV4m0e3l9eXZFgGsE+0gvQTCgHWLhkCSKxJvitPIxYC0945KYFd6Eo36CckDuEXM9Hxv+TXzwEX2Mbho8YjmA4yOdBPoGIEq/vWLDUohyiSQ58hom7LzoMI5rqUTftJOiVANZ+9BEWzn8T2/pMlH0pvgQ0toZkfU/+8iZ8/NxWaBoxzIQ0bC6zcOSndjIvV/IJFpfbJCUbdXV17pwkMQ1C6GIN1j+LlkMH8XgMlk11VAWBEMEym6NDPBbj802NjmDBgd14fv57sG0xVpSWmssr7tpQV5qAx+I9BvNaYtTd60ENDExCsx5UuDF+rivYp/N9+sFZcHSaNAG8+tpbkEJ+TrF6OjswvDGJpvoEfn//b5FnKEkbW+FZw/Q63JVFY13IoN3ha8KovZxQ1JlpDwxkcihrxIWo+Gj+02wQYkqlkImSsWpahT9c6onhA0NlrwTEsF8Qp0OBwav1iqBAxBR1X9GDHP3jL76J1xbsQKFcAKwAbNlkNv61h67FscdMgD85Fk5Fh6bTNXZ4TJD30Fwya8i1eNLcg37C3zDicaW7tbCaf1ejiqwNbtKcP1ztkGiaCu0GVNauHujoga7ZKJky9nb2oaw7rKSq2DTWRjBn9EGGq6gBxIJ+qEEFpxw1FVde+k2ESSjg2AhbNBhbiMp9chWmFOA+U8mnwMewzGVwCeKSQoa6gOhCuJGBUz3RwgKLSjMUIcgzWxYWLFqAYWOmYNeH8zDsuLOhSTSYusYDmyayuRzDZc9Tkme/7Z4nUA7GMWLkaFAHCJezaLIjf/YQgDsilORq1MZoO7j3orFoa0iiftoXYBphrF25EgveewObe6ooqUneQCSPu/obZyHVIyP7qYlSucqCAsMUxkuOiyINPTjHNbwoJiEeCXInlBeNvc1D5JpHuCXjMU4JyJ0GAz6efEnMeLVSQoqN3kSmUsLEfzsa377pTuhOCTppi60AoBK7Keqi7nivwfzVy8Pcyq1YRMo/XRGBt6qsK3bHzNC1ePHRB2BrJRSLZWzftBWG5GDNqtVYvGQRfnv3HQgHZNx5xywUCmVGNz6/yoorehApRVM0BFkl1EZUyqFUyHuwZlxR0dPXD003MWXiSLz69F3Mi4TDBGlpWJs324wcgilKYm4XEIsuXMOlTb9h/TpMm3bEQWUVNg4XzRGxJMnuPClbwm33PI61e3X0pwfAzs6h62di9as3oXX8VEi+ZlRI8OEesme4jPZchOIZJn3mFKTWbt0KL5eL3K//leHWlvj4er36++87FhtjgJVi5Dn27e6AIUnoyVXQmymhL51Dpmqhq68Cw5U4EsQhsqohGcEDt/07Jg9vwd63lwArt8Ha1wt/XueezwANOKeD9lE+R80lshj9SkO8KJ+iIrwfMGmjBP2QkwnIflUoelQHKs2Goo9kDJFTj4D/xEkw+srYsHktwnWjsP69VzDpnEsZFnq5G60NeW+PiRWmT9vDwux5q/Hemk1oGzGKFUgEjRSfYDC9uVre2tJikkMIeIbbmELd1BNg6mFs/PhjLHhvDnamHfRVfUKcDgOP3HwjPvnLVlRKVGKzWMNt2SROFwNzPWUWXUSv3jxy5EhUCrlBgTvls94xm6YYek5N/HpViOdlVTjPaJTywypSdcnBUgV1Ek09ZxLmrpiD9dv3Y8n2PiarPJKJ2dqaAfRetBUbuGYSBXEQg/ppsSJkFKyTdpveX/rjA7D1Mk+szAwMoKOrk88zFg6jpS4KSyvil7fP4rtJ0GtRbu85K1p3ym+pU4rgMR0Hiyeo1cF1oMQ/6DbQl0nD0B185/Kv4hfXfpMHG0YOMdx8ITvUEfQvDJfSD683t9Z+PMOlVk8aLEc5r20pePiZv2Lemg4eAqFTSc5S0NIUxBtPXoPh40+GLIdRztH7esMlxFBFRnsui+8FDe/9/p8Z7uyHrnXIQ9BG4EWVVOzZdwCmRcJuDbmygWLFRJpu79GZRbEsBpEFVBUTxw7HCw/fgX1Pv4ny3xahmVhTy4JORjkIwQTsYxKopuOfvCNdZN44rs5YnKSASsK7C29Kt5fgMpSiwnfTv+HTrn6EfQ4yMw5D+7r1GDZlBhNUVCIgppE2vUZif53GwIioxqUMy0KuVMHb7y+FJgW4XzUQDKNAYgYSRih+FsE7sg+qTBuUDIhezcZvvzkWTfVRNE05EbZUh/WrV2DJe+8gmQihLpnk3tipRx2PHSvzyO2qwqLSEOU5VCs1RR5JkNbP6guX3TVNtLQ0CSTh2Oxo+JYo7JldNVu5xHJH2uRapcxaZuqljYSo3kjGX0HbyGZRBnFhV3B4ECt2LcTuvQfwzpo96Ncs+AjNhEOIRxJC8caQkGCP28pI8kFXqebVK72OILIjFnCwkIPKLQ6CqowXH3mAO2b6+vtQyOYRjkaQyWZQLlcxpq0J+YF2/OK2X0ORKbISchDQnPy2SlDf7+e/p3Wn1ITOn3N5cuZUEqJJoLaEvv40qo6DR2b9BF8+7Rh2eMGggMrMHtLAwkKW0wbBJAvz8FhxL+p58s9ao6WrSyiSrg8TU44Kw67wbO47H/or2vsr2LW/B5aj8nD1S75yLG7/0SmoG3MG5+Ua1W9twfyzU3RJtiFmXPSY/1cPdqo1TvJfTcPwXoMj7mtkuG4uyPS17EOpoqE/W4AkB1Ck5vqSxl0fNB7m48274TgBtKYCeOflx7Duhvswav2AgIPEvhEb546uZKke3cbD1aSqzpDQgVQ7NNWQ8z2X5fS8E0FKEmnwybh9v2yQkoRqQxSNc+7GppN/BPX2i4Axw5Hfvxtm8yguVYjiuchnaCN4zdqstWV9LDD71ddw5umn8t0HaPRJKOjjMo1m0R0GDOzsSGPSxAmY++EaaHKUZr3jwUsnobkuiuYpJ8FEEhvWrMSKRfMR9pNEzo94LIkTjzsHi17cDVu3eRC7ZwB0dwOumxKB4U7tp6maw0eMEPCONrM7eYGcZ5SYZWKp3aFq3NRNqYJOUjtKFQzWLVO0bWigCRWWmG9EghFqUE/5YLSZWL1yKd5euA4b9w3wZPdwUMW3vnwKlrz7Ks784pfwyYEBZKsO9FAYCo0gqelh5fUSN1Pi82eGlCWJVHqTEPH78Owf7uc17unpYeecLxTQ1d2Nhx55BM/+6VHk+vbhF7feCdumqZQElwNsUrTfAm5XD527lyKwcMaVzYpyM017BPr6M5xivf7sA5h8+HCXlRe3BiGWm4cdVopC6+TCYxaqHHrLm8EykyjveA9voiRBd3pNmvl1oL0X9z35Jj7d14dcmaoT1J0r49kHvoPTTjwCgYYpMGhyC6Eq13Dp9Qi91g49F4TgP5eDatllrmbUPudz8tpDI7f0/KzLxSBb1iJTKUblG2gRPCYIoWkmjwwp6TqyeQ37enqQyxmY/dxDwOLVCPz5A5gEAWkEDTUp0NhN13N7hjsoYXNv6ET9jjwS1VXI0KoMlYAczjW5W4T6GrmGKYkB5pA5V4r+6UbseOlNZHr7EPjFldi//D00nXAW3yFALIjDBundqMzzvASVaNPdcsvPccIJx2PSpMPF/Ct/kEtgsWgQYWJ/HQV2tYiySZMdbGanT5/Wgrpk3DXcBDas+Qhrli/CivXb4Jg6vnPxZbD3R5DeJ6Zc8M3PPPUPRXSXLaVxK4Q+6urrheCdWt34njlDk0VMQ0MoFEChkEddHT1PRBVTozUTs7CIzIKkI5GMIOgXih+WDdo+FJw8Wk9qwfxF89DbX8Vjf5mHlrY6nHPSDMx56SWG64c3xlDvDyHZ1gC1uQmfFVR8mqEZxUIn7m0URkS0nu45UeHMr0i47gdX47ipdFcGEz09vdi1ZzdHm/vuvZcVXS8/+yTSvfvwy9tmQYy1IqcllHVkoH6/mJfNyIxHBymMSLgk5DLZPAbVtJGjMo9s4aN5LyEcIsmoGBzvGS7fQ6laEvk3BQ33TgS1UY73xb8wXO6G4vsECRRChjd37hK8OG8j9nVmeFwxlaLojhMfzv4ZRh52JJxQGyoDNClTnINXU6Zq7v8Xw33lge+x4Yq8hXprxaym3nQO5SqVJGQUylWkswXIaoA1t+OGjcANV16GjsvvR7RiQyGFC3kaunuBIyLloMzLrft5bCVtANq4NLOYWU0yWpe1pIgkanOiBhbwk5TSHSlDdxzg+wYpSI9MYuLDt2Ddt29F7398Ax2fzMek2LoysAAAIABJREFUf7uKo43nyUhKRyIQik7UIUQRi2vQEnDnXb9DV15HXVMTR8CGRAz18SCSYYVvp0JN33UN9UiFowjTqBufgekTGpGIh9B8xMmw7QQ2rluDNSsXY9G6nShYPjzz61ux7m/dKBXLyJDTc7tQ2Ou7JVkel2LbSKXqWHBBtURyWNyd5IjeUxHZ6H44VdTVpcRgM3dig2hXFvmqblSQSoTgUwzWM5N6jYYDyLaN3lIZU86fgtmvv4RSuYx0sYot6z/D5s072KHQrVbaImGMTcV4cuaxXzoV7819F62NIxBuGY0NPT1or1AUUOD4ZKh0fUg3yt1TfvzsB5cj6VMwceokVj319vUxYqVzpTbNx558Cj+/+QYM9O3HnXfcC10n0YmQ/nksNZ83OW5XhEIbn/6eBBqeSILSpnK1yudAfMmmxX/lu2IQt1JL4hBTTQ0G5JQFiVMjruD+X1doUSv+rY24js2pCDsPEn0YOq6//XGs20OTN0WLKBXkaDTQ/Jd+hpbDz2SupjxAY3CH6rfEy/C0i0Nu3FVLDR+EAtzIKhx3zQG5XWMC4g9pGWoHWEh/++1VDrfEmeT5qa7mZ8Pt6s1y5KAhbDQXuT+b45IPlQN+c/vt2HjHn9DywU6YpHnlOaokCxNpB99gxKt7eY3i3GcpciVSp4joKHILL+IO1hm5Id5AmObluvI3rrdS2YRQgQ00Ln4YC069CvPVAdjTG3Hh1TdCc6EdvTcZiSB/dJEHsXqI2GMHn2zYiuf/PhfR+ibEUg2CuabJiQrBOIdvSiXRBShloCgmjhnbgu9fdBbqUjE0H3ESbDuJjevXYM2Kxfh0XzdOO/NsNJfqkN6pIJ8roFwSrX2skHLvS8T5tmEgHokxk025aTIZ5+dwq5/bZsdyTa2M+oY6Lp2EgwICewIVT95I+W00TPet0aD6RcSgzRcJBtGRLmL6t6bjuRcfxrixI3HLLb+FZft5YgjladFQGHU+H844+WjUtdRjf1c7OnbvQ8L2s6abjC+YiOPEiy7Gg6/MQzAURdhvY1RbIy788uloqY9C8ScwbORoXlO63SfZBMP8aASf7dzNDrF/oBsPP/QIHJvu9Eh3InRvRObuUS+F4uvqTj6hurSQPorNpBni9qWQqti46G9s2AG/qLXSg9YhmyVmlyg3t7zDrYuuJfDGHyrBHZpriroveE9yDm8RJ2Pi4usfxq7OLAcOErLQq/3HFWfh6kvP4NuMUJ+uWaSJk2Ltee9SfuuKfw5ihz8naWUU+N8w3EHKuqb1mt/v5fu+6/BoSy5TUKRUeeGyuQqqVBCn4rthIpMvolQ1MXnSWJzzxTORu+Be+Gn2DhkJyfP4s3gb2k6DD8/w3FGuRDTxIGxvzpNruLzQrsaWNi+RNNQB4w2sE2NT6bYaVHpSoc76Hna/+yFy23aj9ZEfYv3WPWgdNmJwSh95cjYe8uDuhAUSB5BEngaSjB03fLB5W6ObSeUK6M6W0NWdRldfBnu7+pGvVvkeMOefNAbnHjMKsViYDde04ti2eT1Wf7gIAUfCzAvOx5IX9kIrUBsXOQshuqCITw/asMSYUjtkJBgWEZSaHywDca59i6Mi50kbNx4VZZ5KpczrRPCVmFeqkVPkoteiOzqQzFNyKpAUMaKUcmES3g+UTEyaOQVXXn0F7rj1CqSifnSmy5g7bzXmv7+SeYgff/+7aO/eyY6G4N7WjVuRCIYRsiU0NTdg5NGHY/WWTxGoH43DRzYhEbIQRBWth02H7I/yPXubxxzG150MlwYIUB6bzmQwefIkrF+/ETt3bscbc+YMGi6thefQyWF7hjuIOujKMMnmZm+OhAoNNzctHHf8EXjmtz/jyZWkba9FdMQXsO/9XxouGSbde5mOg27fSRNGv/6jPyBfpuFwpA2gY7Uw+/fX4Jijj0CgfiLKxPBXqTQ3ZLgUlYX665Ce2/+HhkuWRXeZlF598FpupKc3oy4M2lQ0y4dCfpXuuseEEzGeOuh2nHfedgc+/vHvkPz4AE8CIHtj76HSd7X26pIbjsxMH32QekbIzWjciuhYGRwOxtIzMUCO2GfOrWoWgEem0hj0ACm5AnDO/wKkyeOw91ePY/z8h7Fk3SdIJhvEAdAxU47Jt9uk+7WIIWRC8yGc1D333I+jjp6Ok086Hg11CTTWJ1FXnxDsNwlFJBkawSTLwc6dW9EYqqIhlUDLEV+Aoddh+9Z1WL1yPoaNHoV4cSz6t1aRzZdFlGe45E53cNMB8mU08pNgqjhEGv0pBAGJRIJvjE2GTvXkFN2ylG+aJoyUYCRFFoL65XKBG0AYurqN5o5ThuqTEI8HEY0m0ZfRMe3iqbjm2h/jsDFNOPfLJ6AhKSPATRVRZLJVbNu6DTv3tKOvP8tD4j7dvoenbM78ytlwAg727tmBq666ENt2tKOkUeuljVR9MyLJVoTCCVSrJkYfPpmhPbVxljWhWuKvCwUcaN+PbZs2Ycvm7dCp0lDVuT3PKyV58lIBB4dKTN6m9/gBru3aDh741TU490snoFrSWdsucnBxl4F8IS+kmO72qyV+vNzW4z4+rxxE+zYaoRo5NTU4mLt4DX7z6LvMNg8y7ABWvfwTjJh8HORwI0okc3Tfj3TbTGqR2o3aVGv6bcV+d8VGh7TmHSSo+JyWv1qozOvi1oJFxL33KjEBgzYKTwChhmQaOGawbEvcmYzIFgmJRArf/NJMtF94F2waRVozlsNWRH7JCh0XpQjqX4Wf5zKTzlnh16U3pp5Nd6KS2MjEDjJcF1MXPCUJRyx3tArDKVlCOBZGaVwbmm7/HrZf9ksc9tjN2Ez3EyIn4d48igdeGyaKxQJveu735fooMc90v9ddKJbL2L51G49E0S3SvgYgwxT3DQqqmDZlIk6ZNh5/fOJpzLrpSjQ3pDBs+inQ9Th2bN2MtauX4vwLv4Flz+xFrreEStXkcyAvLfS34jYbDPdpNCmL4l1JHzU4KIpotKZzClJUtZBKxQdrpXSlquREDZ2b3akcFKF7tsrkBN2eYZ6aaBAlgngyiFisDgMZE0dcPBnfvfpqKJKFyy69iG9mXd8Q5FG4VIMncQSlPnmN7ujXiAULluGEk0/Axg2foLuvG3FVxxdPGEN3H8KBjjzau/qRaBwPNZhAQ0MzO+ymEaPYwZKx0qhUijYEZTPpAaxe8xHynb3YuHkr3+FBqw6Vg7xI6+X0XsSla13bm0vPo3SBHvNeewwtjUGYBh2vN2mSFFNVvpuBUOQdXCUV9wcWZsOTNEXB7J8EGCStJGfgkYWPvfgPvPTOBkZF3iMOA0te+wnaJn0JUMIopbOD+mRvj5Y1ocOujbiC63DFF4ccn2e4h+qTa2G21wLLebB7D2H++qW7r+S2Pmb73JDJ0xFNaimjmh01lBNDClxwwYXofOQt1C38DDrlIq5HooM16Z633niaGsMllVmMJt7R0bu1XVG3GpoEIFg4TzNLKllvSBqJ/N082O2fpIhLA7H1VAL1L9+ODedcj8SFZ0O+9DR0D4hiOF0fJr54lAz1xgqxN9s0T3OUEY/IaGtOusSYmJ5Bf5PJVZDO5LFp41b059I4bGQb/vzim3j+nmvQ3JBE27STYZhx7NiyFeEAsGdNHunPLKRzFaJAxYA6Zkf/D2vvAaZpWV6Pn6/X6X1mK2xhC8tSpCpNECkaRIiKKGpECEaTGFvswW6MiUaNvUTUGA3EgoogVXqRXVjY3ndnd/p8vb+/65z7eWaHDf5y/f/X7/PyYnd25pvvfd/nee77Pvc5567Okfp1QoZpZ2uSNz4Bps8Uk3MkChcf9aukLcqczpcRJC0Qqa+yHdFET5eZk0s2x7GjAmPYTuFxVEY6E0Z7Wx+mcy2sfc0qvOb1b0YrKOOyV1yGJYsXorMtivZsm2h7nekU0tl2RJKdQDiLeqiGZtWECZzAMDP6LKKFHRrSzLGos9UwxvPtGtZGVgkdL3sXLlHGwJqYLUQvp8zlpnHfA/cht/sANu/cgUKDtEBGbYciO902Nyb/L2TZtQx9EOF7Mf1n+s1rvP+2byOTpjcV+eVHjMHp4czD4k9tXLYIvcPin9q4HOotzrTQ8xre8nf/iKf3GxjnX9dceDw+9u7LkV50EoJGHNVC0Y1PcYMD6EzqpkL8v9y4mmPsAUy3cXXYf++mNyriCjmjEXeViCbnzhjTh1pWCr4TkTje+JprsO3PbkK8bJpXOdITTSYSKmd892JYd9pY/lwqEhNYpAfFDyHp3xEfKv4b00Iflf2pK8DfnTSKlVqknMERRSQbw/BvPo/Hzn87mh0pLP3Jx/HQkxvQ1dNv6bDT5Jar3LhszPOhW7pNjPCpDU/h/ocfxdmnrsXKFcegr7sDwwP9yKSSqFFTWq1g4zNbUC7PYt3q1Qg18+jMJDCy9iw0Wl04sHcvGjPAhtv2oVys2jDtqi1e/g4PRrGu5QHCF+VgbOewbJBDZjyqw6RULmHB8JD8kxlRBfTxMGUJ0mxq8bLO7ci2SeqXTFEfax4NYn9HCMxwpEkL3b19mKrVsOrCU3D1tdci3hHBxZdcgHQ8joHBfoyMDGrIeCKRFuHC6249+OWf/9jOBxCrjavGIb2QQpJqPYotB1tohNpxzHHLNN6kt7dfzp78OZFMmk3kCtMoju/ELT/7DfaMTgrc1CesmyeTRSXvV2aHz/ya1QcSUmp17dEQ7vvVv2jTUoTBA8Be5jEldJ4JqaslSRDxLUBRIqVNdlxheWs9v6+aITDFz84MslHD+W+8CYVGCKEmJ/MZ+v/Aj96PJccMItK1As2CaaT5rlEHlHnRvI+4z4/99mntoLXfPT+d9z8zF63n/bA3kfNtOZJTcrOzCH3rI1dr45oEyfSbQv9cjUV9bDVo4lWvuAKJ+3eg8tXfolzhsOqWLFcIHinyOlsSF/BslksohAy9mWnpwtS4BbFlJMTWyA9nq8oeYcvpK90GF6+TrQJ/ErOdIB1wBIloEvG2BAZ+83ncdcENiNbqOOHBr+MXv74DI4sWO8M/A6c0woMR3cnnWAs+/dSTeHb7dmzYM4njj1uJbCqJamEaq5cMYO2Kxdg4VsepKwdQZe3UKGKyGGDl0gH0ZuNYuO5MlMpJjO+dwYENeezeMIoarVnrAaanJ+eQZInznVuFZ+yQaMD0K0GATTrcCBrNGrq6utTKKJeL6t+ypBDKzxS/0cTM9AxGFow4ZRFRaLPaoVuj2mkRWoXS2qaB3v4+NDmlYVEPPvrJT2Dk2AGcfuaLsHb1Wov4PDCj1NqagyafA58/a+tcLq9NRET/0NbfIlKn/WkYyWQW1GLICxsxHJyOonvxaeju61Imtn379rk+KNfR4Z2PoDM+gV0Hm/i3798ubWpUm9D0snq2nPLoDmXeE3HfSXF06LsypGhcAN2CgR784gc3CYPpbOtA1fX9mYTRUZIZCEOB5y2bx7IbSSLFljNadwHK00l9nCFH2Ud6thbOvOp9qJEp1YqK/94KSnjsJ+/HwjUnI5TsQok+TgoqvOfmeOqHVv/fNq5tWPutz0Odj/r70a0h/71+MAFLE23cud5SyBrkmprt5nmSh3rM4mNwxZVXYfMVNyFxMI9yhDR3jdIzxY53p3cnmZQ1gdmhhOsEYQIEZAxxwyLkRNQEpqxtxF6ZqXNss1oqaVHba0G5+Yg0c1GlYmkk2xPo/eVn8ftXvxvZyRyO/f4HsTcGlDkpQJC86TvpFkG1E69ndO927N+9C3fe9RDOOvN0TWmgFLGcJjlhDdKNaTQD0h3LSKbiKFcpK2vg0FQZq5f0oTsTxcDKU/DcxlkUt7eQH6/g8MEpcGod20iVWlHSMtb+vB7W5MpmXJSx4VQ0SuNwZx5CQAeBKKlDGGHJ260jJZaYWfLQRYGqIbUbdMDVEI4Ekglq0gLR5gR7rsyLqiDvOdTfiX2FGRSbdSxdvQixBEn8hkgbG8oOQLHaHNWO6b1F2zqmp6dQ3H8vx32pHKBgX44VkhE20azk0X7shagkB+R8snXrVr0v21FMmw/veACHJ2Zw2gWvwdo1qzA4vEBYSaRhJRmvSxFOuAPlfkckfWSzsa7l8+PUP94bfvZjFmVRJZ+8JQs/A/doMkh2XIuHc1VMOO7XeqWEajGvsqXZpJj9+fFPQWWeoES2SS7D2bx9N66/6WaUajzsSSwKY2Aggd999Xr0rXopmmHSHE24ImN4d//oejL/PV8o4v6/2Li8Z3KO/M7HrtHG1eZl6sshRw1LPfggOX/0pLUnYnVyBOUP3IwCpVPhEKpEbclJ5hnujjAPIvHWZhNJoau68X6AsenEjEUTtsl4Qu2YsGmh+ka5a09pELmrizgtLm5NegNzsuj+wXtx/zv+CalDU0i94XzEr3gJDu4dg1YbT0oynypFjO7biX079+LB+x/FqaefiGUjWVSaKUw1ouiMtHDuRWcgGy9jyzM7EImnFfXa0hFUa0ChWcIdm7vwjj8/C0G1iR2PHEZ9KoI8J9FXgWKpigpBiQCoFHJz4BRjgJElzMmCC1GqKkaXaEz96I62jO6B0HUnvZODR7lk8j2SUFJ0Z3JSSNrjCHmvIx0nfZAHBAkSvCf8piqGhxei54xj8ehdz6J/ZSfifWkkmeqKceVSSPc8dLAgsFm3bEXVyzg0MYG9G+9DWyyHRCyJRNJ46VznTOtJ8avUm+heeQFqsS75aG3e+Chy4/tQL09r0PSrX38jhkaOweiuWVSmSqiXWwgaYSTCSQcSATVmbeQ/Wx9HBxEPEpZcYs0xatJ1UzOrbAazZYYE/VxfWzArwTb+n7RrJ1GMRhBLcqRpCBEePHTWFFehhuLMKAq5GTRKBi6RgJXiemlGNIPqi9/5OW69Z7MkmUrqQ3Vc/bK1+Id3X4u2hSehUamgXLaNKwsn53c2f+OKduvCuaXE89qj7utHR1wf/Y+Oxv77+F+uHw6RV6bCGtejwwTD6bzATgM3pdDRRh03/PW7cfDyT6I8OmGm300OZnD6xjDlbNbw9myYGNs54pG63N6hajYo2kHjpInF4oqOCTGirKbWAcKmN6ODU13we+gvNIe+hUNoT7Uh8aXr8dQX/gPRzXvRXLcIa778Hjzw8BPIUGGEFg7v24Otz23CHb/9LS6+5CL0t8WRbx8GFq3D7c8extKggPddPIxYiDV2BZs27UGUJIZ0CskUS4YYRpaegFhyKWrUunYPIRxJINQyMrwUILocuyamv6qtXKtCaKZzYWRWIeaXAqlzkaCG2PppcyNLXTFk0yO4aOmNWaphfHQc+zbsxaFdh5CtAbVWHQnqiNlWUx+9iXC0jmUnnoCR01fhrp88hMWn9KOSILMqjUajMufQQNM1LgJ+1q7OTul9efJs27oZDzzwAFr5fThlzSJZtCayUSREkifzDPLLLlXr6Ft9EZqJbokAHrn/12gWD0jBc/3ffBj7dszi0MYZhMoxmbrFIgnEogm0Yuxx2qTCZp0m61XDNgIudIIwIsJqHXBTZ2iUJ+6xH89iYBEzKfWB4zHZBbFDwVKDmQxrYvbGs9k0SpWCEytwsmAOQbKEdGcYi45bjL5Fbdi+8THEawXEU3EBs8RrXnfjp7Fnqq55b7RbCocS+P7n3oALLngJQulhFKa54Q3V9mWcNyb0m2+OSDS3eY9syxfasEf3fefXv/77eRhQUTU+Pm4jbpkqe2dEblxGXDOlNqeGNWvWYH3bEoy/7WuohWtqEXF4JS+S6CKlefyzr5OZdoQbHIdxhMblp5dJRO6dLlwkFuLqmE1e6eE3rgqoUEh1sU/ptEVcxE1+8W3Y+NVbENm4E6GuLJbfchMeeuAJNMINHNy1HXfcdjtefNrJGBjuFEmkmBzCg6FVSCfDKI4fxKcv6EQiYY6J9InavWtSiHMknsWy1evQO7QS5UID44encHj3DMKtjJz0GXmYlgXse7vDlAswVDEBPr/Eg4douVwe7Bh1BAu2TCylo6GYvJeUOpo3NR9QNmNDuwXShKugq3UoHsbgwi4MrBxGOEjh6Z88hqlDo5oyoEjVaiLbHsPQCauAgSy23XMAx5zRi1y4hFYoiliUtaWz0E1nlG7RhJ7kiWwmo7bUX739HTjp1HUY7O3HxN6NOO+01UhlNULc/KF4knLj1uoYWncpCi2qfkJ45rHbUchN4Lrr34MdOw7gwKMB6rPMMmKIJzkegrUr3TzswOJC5zrh1AFNwZCYgCouIpos11rIZGn9a4wrDz4RByFZhPeUG5seZELwJcYgDbQmmihpsfVa1cayhO2ASkVjKNXKRvmkk2PvBE695HTM5HehNXtIffFys4lXXPtJ5Ko0g6dpQ0ssugf/691YfNwZCCIdyE9OIuxYXv9/Nu4LtYDmDvIXiMZz9S1bqAHU3hRH++sfulpjNj2STPiZtSajZritDW99/Zvx4OUfRv9YFWUO9Q0a0qgSU+OLaTLBKaKfYrQwySYfmYvQiQV4E3giakKd5CG2uAVUaSaa+RboQzohtUcWiTSL7ujkfiZcCCGRzKDna+/C/f/0HXRs2o9qGFj/u8/j0c3P4cdf/yZGFgxh7TFDWhCToTZsjS/BWGoY/ZkqTurKoK01g/VdeRndNcNRKW9K5SaaQRYrjj8NhXyAJ+7eiWY5jmSQRTJK07KyIoD/TLwU7+Mk0MWl+joI2f4IkRTRpl6sH0rFQ0pqGA0Kt4jryfY8LAlUkQ7Jr6kH7HqWjteGYpBDrDOMky9ah5n903jqJ3cp6nJywPpzTkPn8Utx/2+eQKsUQd/6djRTVHwRjmiJWcWDktzzvr5+/W4DxUr45Kc+IVLGmtXHY8XKFRgcHMTeHRtw0vJ2tCeJS8RkYkcTOtIQB9ZehUaUHtoFbHnyTrz4nAvR33ssHrh1G0JFNwhOPttpM4j39rFaNJR5RrV5D48ddqbvtBsS4VkHisz+3ARGmRQ4RhXvC1NUlnEkPtAhRL5ijYZkebzn5KdzQ+vQ9JMfKQ/NsvVWNgAwEUE9lsOLXnk8xkafQZ3jQWeKeNkNXxDhwzyom+iORXDHTz6AoZXniAtQIoAXCsReYp7N0sZrjL0HwP9oBx0ln1fsOYqk8UKRmBuVpRS/l8+N4KE32At9+X1XBfkCJVGqpFwqA4TjCbz+DdeidNcmFD/yY9RpoK1ZKnVUgiZqPI3omsHZn0ELiSgjp9ViVGjw3eYG/BJVZBokiVgY9UoVWfZ2XfQNmnWxlXSvnG8sN65O5mTK+nxOZmZ1CaV0WQz998dx719+Coldh+Vn9MiKOFrr+rBquButekH1y2TbSvyu0oMgkkF/OoorhktItKYxsmBYn5uACXW5zAZqzXYsWXkidm+ZwdaHJxEPEmKRifwgIoQNreZnNA0zU/2q3TkN3wqLqcVoy4g8ODik+lcnqrdYEXKcVirsWVSMsvTnGh4Z0kMi+urJCfwvFzEXinjg4SjqdeZGBay+cJmMCh7+7s/R1tWGkbPWItXXiQ2/26nIMnBSL0LtDVTqVZvQ4JhoKSmh2sxxolHRDCRGP1r5DAwMoVgsoVQsI9PZhf+6+WZc97oXY+FQCrGALpxllGsVLDj5GlSDMPYeOIzKxG688rLX4g8/34RosQtTM9OWlgvDOJJteDCK94MHGw8SbsDZHDnhZpFLbTP71myRzecyc+MKvHSjZmy9UOJY0+8hMkx3UOv/0kPM7GR9RFd0VvvGPLzYimPWkRho4awrTsOOZ36DbdsP4C8+/E2Hu9iOeN2lJ+Gjf/s6tC04AdViGZViSZx2yhI1b5FtR41OsbzghV5HGI82GfKFXkdvXMtgW4hHzR2T94Ke457aGvrSe66aG2wtIUsQYMGCBbjqytdg9y8fQuXzv0S4WBYPuchZIZzFE4ZQ5fkblxvS17UaHiKKoYnHaRKn9JLIKf1wqf+UCNqRwnVCBjYJ0NW53KyefM8Tle+p3J4pJ10gkiks/cO/4t4L34n2XFluE5lLlmPy5Da1UHhIFDIj2BJbiH2zUVRTKRzfHsKFg6PoiqYRontEKY96JIUo+UHNLBYvPwObN41j15MVxOnWWGPmEHIjNG3TKhJyKnqCdVtMOmSypJQ5hAJtVG7c4cEhM+d2TB2zPJUd4ZEeYxh6H24a1mVqkRklfq7eTyWSSmN57eZ6yHlABiiVG2WcdsUa/OG2u7F8aAiDJ6/AH371OIJiQkDMglM70cxQUxdIqmhtmADt2YxcHSbGJyQG2Llzp4gqmQytUt2w8loZPZ09+Mb3foBzzjoFs4f34KLzT0BAMghaGFl/NSrNAFt378FLT1+P3c/mMfF0AzFwYqD5dHNyIfvFVrMypbeFLvFFyAzQLdMiQ6wsVRb/3ffxGXG9nlrtaqeMkiFBzAQRsrVNJPRMiMlYKspWkrH1zB0zhnQ6g1yBEcs5PLoh6mwFHvfKxQjFpvDFL34B37rl0SMbNwC+/Ilr8KqLz0couxBT4xPKquZvXIFSDmT9U4L5uUkTDoQ8OuIeDUhpDbjsjbiJ16ITmCI+0NPTjdC//M3lQaVUAZdYR7oNl1x5Ffomm9j0jzcjtYXeUzU0WpYYS/3QMgd+3nKf/un0m0fnkku9NquG3ZieViMOzU+XD0fTRwlaOSKab0kxCul7mSI47ylRvTiPxonr+Tniqxah55sfwtbz3yn0mLDFeHcdnTecIiBmJ3pxqG05ikELhXoCK3szuGgxhxGTwUPheVS+WqEwD400+oaOl3vjY78aBWdV2pxdI6aoZcUSwpl4+2xCEYQaWDXjAY4rpTXr8PCw0nn6RstbqkHXCjOCZy+OAArbLpwLxDRWEr6uDkUfLbzA1CqKtGSJ1ex3mzyR2s8kIrR3pd9UuIizrj4VpYkxbNk0huJuShmt5ZJclkMrxjQ9QDbZgUjcrGjp7HF4bEKLvrszi/EDBzBLhU+oimxbO9raOtRZYLP/jxuewvihcaxYuRLReB0pjcoMsO6Cq9UJHCBIAAAgAElEQVQymZmewmknnIG7/v0pRBspgZoh9toTcYyPT6hdxA3EqMQD1RBiUwlxbXlQjwuSm4ByT4/K8qDXuhC4GTWXlgZlf+zvGwmDmYW8tJwzpt+4mk6hEbCGkZgtEbM4Z41LJls8pjWFTAtnXrMeZ7zkbOybkHjYDuJoDPd8751YftK5CIXimJmeNhFNxAziuUZZNhjZwzJB/3p+BHXdE/fPR9JkI58cDU7Nj8g+TZZE1Q20Y5kT+sxfXhqEolG8/GUXY0FXP7Z88gfIPnEAiLG9URJqR40tdYdawMT/ND7DFrTAJdUtR6RTcdbIRN48b5OFPp35aMjmUmEvPPDjNv2HZZ3X2dY+N3PFEnjrmc3d0FAU3R98ExpL+rHv+s8beMOJ6h1RhG5chkIrid80jkU51g+EGzilK44Ll9MKLySHBdY4HBAtCh5bK23HoqtrBX73H88g3ezQw+Tm8iNQdPKLJGCgiGbUOuN3Xg8JKeoNIkBfX49NDXRRmJvWxlJwIcXQ5JAzDTQzJ0GK5tnL9SMuuPDoDOIXhr/H7A8zmvO9bJxLSDY4QTSBkRd1ITWcxnP/vQNNKoYcQr/otFGEMtMAUmiGqkhEF+PAnho279yp6fW7dm1Dd3saixYtlJa6LUtKJQ/hMA6PHsbuXU+jWi5icjKHgYEBtHdmZLNZyE/jFdf8lVojy1Yci8d+uxWV3TGZqzPzSZEt1uLIy5yMGFiTGnvNi9RscBkPJj5XZmDcyOxZlwp5JNlXdb1e3Sj18zm3iOJ7+mZXnUtkTPU5D1jzFPRjVRtKhXmfaErnN69lR3Xpodkvnxu3GY7hhCuX4ovf+Ta+9u3vuh5zC7FGHU/c/gn0H3uuDO/JWOIr7twcuaY5YcOCjnWXj46e8xFiW7+OeDLPLfOFIq7/mth2kTDGxsYlmeTfOzs7ENp730+DdCaLrR/7LhKPbEfAcQrxGKLsJ7YaKIUDzX5Viurm0BKv4wf2PFOdmvOkSxoxxGkFvi/bbBmpgIQNN6uGIBYXszyC3Ga2E9R0uCKHa2atG6I9r5iPdLZj0Z1fxYOX/TXaxnKgElgT5RIxzFzei4cGT8CziVWoVetEvpCuTuLCkRZOXpxGF3unjiLHeB8JJ9C7aD0ev2MclYNEP81VkadxscjhXdY3thnABKNs4zI6yhSedjq0gG21xCUmMOLBJ14Pa15mJNzAFBkImJE1KRddWUZvZFzRelSCeicwn9u4jv5otkIhtLe1G72QJu41m3JYQA4X3XgB7v7GH/QZJUrnwh86jJ7hHrR1pBTBSRlsNCM4PHEQd999L/bu3YXwzKSM87bt34cgTAM3G6FB293ObAsz41MYXrhIRu2DA0Pyj56amsAp57wSmWQCQ0OL8Pt/30YTSW2uNGcAhSKqH3mdowcP6cASycH1bU27S+F7RAcRa1NGHn7G/OyMwCZ1J3g/2G5sNJFMWDuwWiObyyYYWDZk9Fu2lqjx1s+xBEnSe8zsivje9LYiqNTb06PNG43xWVuGw2fYd0oGQ6tH8PEPvFeHAUe9DA924UMffiO6+46XXJMHC78/6e6RDPfnlE1cVV4PfIR+8T9BJ2c4f9Sk+T/VJlJLMBwSHsHrZ7Yl7fDjb7ouaN2xUYN6a7WyNgwL+UqNIzUomaE3Ygi1SADKhllnJTvbEe7IIDLQhXR/N2Ld7Yj3dAmsaRJYODyB2uPbMPHYs8iQjsaUpUrChiBl45UKKWa/17ntuIgtNJoqHl27m+cTCSPWDKEWbtIJHCt+9yXsuv1BlP/lZ3pPotriWUeB8RdncNeZr8e2mTriLT6YCBqoacpBfnIUo1u2Ij27F6evW45Tl/Tj5DPPxvFLT8bjvxxVRKsVCTqZCwgXlmeqJOOM0uZIyDRQIzUpgo+GFTm4YJgGcwFp0gPvm4EGQq40zZ10zqgza+fw62RMvTljLFUE1nChOeWfO73JeGqoDibSq1Nehx9TXqbzYYQTCSw/rxfP/nE/GhOMygROmug8Lo+Jwqz6uByhOjDYi7vuvN/8nQHs3rMb9cIE+jvasW+sgqo2SgTFUlmeWSesGsHCRUMY6O038If65MIspmfyOO+yq7BwZBjbHx7FxA4rb1hrClGvtnRNqs3CIYwdHtN/6YU8xyHmMvfuIPPMAhltZ2dmnJrK0Gmqd/yMIf6X78FDQUZ8bnCZzdYN0CZdrY0B5YHBTUy9LjcpTfdsdpUNPVOZ4xVunU2cfc2peO97341GuagM6MY3nouVJ52JSKIbs9Mzc4eFNz7nNTbny/H0TNxIl3kg1PxRKKZ0cbFX5aOjP7qRKEfSZJskwetkn533ngc761tluRte8cYgTOJ2bxtiw4PILh5Ez4oliA/0IKDUjNGJ2A0RPBb21SKSDoXNlUuIFmuoT+UskhIFI2gz0I9IbwfC6QRq20ex7X3/itkNWxBiZCKn2QZEauNycr3YRWwhEYBxHj6+leRPoiDKTR7F4q++D5W+Lmy5+iNIShroke0AzWgNtXOX4K6zLkYykcGuXXsw1TmM3Ng4cvkKipNjQKWIanEGqWgYX3n3m3D6iSuw4fdTKB+MolTNIxqwjmqIoSKLnURC/UHR3yJEdFl32onPGoosJ95QooyVkknQBMTQSJ2UT5dS8+ustZjCsfZltO2l/pe0OWY3NTeaIx6VD5ZSMpdicuFx4xAp9TU3nRrIGKpV+VwiCHdWccqlL8J9P7wPcW3cFtqX7kI9xujSoUl3iXgffvGL2xGJBqIVHjp8CDu3P4flxx6LHXsnEGVUk79xSZ/vjJOX46KXX6CevDjfrQAHDh7G/Q8+gnf+7XuwbtUJuO+H29CohUWW4EHH961XWcuaZJGZBaOd3RPLKNQCc7OMtZHmAZK8l8YQmhE6LL02HSBr1TmXCsM/vJuGcQj4d66neCImuirza1Mr2ZA1yva4eZUdaoKCpaCMvk0iJJEAZ71hPV77xrfg6ac3IBEK8Kuffhgr1p1HiY2ki8pEvP0OiSBcz/Ook36UibKBeYPc/yTpQmCVi8BCadyGdoeBzZ6mCQM9o61t2Nvbq4MsVNz8aBAlW6reQLFZRf3gJMoHJ1A8cACNfeOo7h8HihW01YFEyShq/H5uVHoReeYo0UQ9DGkDNSQIhZ4U+j53PZLrj0PjqX3Ycd0/IL9/FNVIC9GggYBEDbGJGGEtFQ3XW9b/dRpcAiSKvuEIlvzb+1BdMoznXvV+pAnkiDUUYUmmGTitSAuVpXFEb3gdJlKduPWJLVgzMoRFmRB+eu8T6FlwHPYf3I/JqSl85f3XYXEb0DuwDA/8ZBtaxThK9QpSkagE9IV83vTBjiEjLnHDVCxWo9oCZI3KTaVIosmAPO2jQpsZidOufuMjYQuG7QsuaAJYQdMDGxYhuGjzhZy0uXygXtbGRc/+rlEnnS9XiykkQas4CuUmcuVJXPjOF+O+7z6MRDylmvxg7RFUgxksXdSD3p42pNo68atfPif8gqNhxsZpdhbg8cefRM/QYkVlCk34+fp7evHRv79RSp9GPauv0VvqmWeekoHex2/6JA7tmsahh+toxlqyzJEEjwPf8pZ1SCpaNwEBN7TfuGrvhUyJxsORm5cAH1+WxlKvTTKLlWjcvKQt8n5KJSN02uSZYvjxz37gnEa5BhpPyvfnUG/+Pg2Uc9MgmQQJT9U8ZANRYqE4ll3Sj/FaEa969RXoSSVxy83vw9IV58mMPed0wb6zwc86f+Nqs7oZODqc5m1cX+ce3bv1I9TtGv9nes2Ny2ucnc3NXXdfX5+yr9Dm5ecHbOVIhkeYnWJ02qW6KQJmim3oHm+yRyy9IZbvzVH87j+gDUI2rx660U8tG8Sx3/kAKody2Pu6j2Ls8G5EeMCQVyYbbsrd/HR2MmysnURieoI1SiSMVT/6LGYSUWy55mNIVmpiO/Fw0Oeg6RiF+OEmKovacOjCfpSDFEIa38ETNYJnn9uCVjSFBWtOxFvf8lY0y3l09XZgz7NFTGwMoU5fI9rHuBSYD51/N9UH38FNfRd7xxYlI65GPc61tawtxAdBAMWnYhQFsC4hH5cnd09Pj5kJcNE5/2iJpVyflWZxdnABhWJOp6zIGCQhubqfMct8p4FimdMRSzjzTevw8F0bER5voRkJMHBSGxBnCkneNr2CiyiVCxJS8M/ymZ6ZwMMPP4zp6SJyRdqj1rFm1XJce81VQCihNLNcsYHRBw4ewMaNTyKIxPHtr38Td/5gE2qzTWTiaYGXMqCnVRCZd26MCwlRfmqdoq7v73O4tu9E8P46je6R7kJ07h4yc+Gztt6mn8hgBxjRaCmaOKZlbjoElWZxgX6Msha5jcQhQoZYpm5Gs+u/xmMhtC1I4ZTXn4Qbr74SSxd248Z3vBEdXcv1zMj8EnCo6Y4WGXmQNI8yjffPf370nNsXR1navFAk9lHdZ1xcg7OzU4jH0+jKtiOZjeOhDbsR2jF8WsDFwyI7iETF9+RN0DR417f0fsg+AglPcnUSf5YEhQa9drxDvktd+MsF3bdCKHTEseTXn0e9Auy+9K8xeviAicrZD9aUPWvUk3qmjciNQWL1QD/W/eJzmNl6CLuv/wLitYrSdvPCptmtsd/VjkED09kQUu86G/UgpgiIUAxVEtejcRy/9hSk27tQD0Kq45YvW4E7b96K+rTV2easT1vXqk1m10gQWr2S8eVsNx1pnAuIG6pSKllaywdaqwosUvrbNO9gno6U4VGXq9qLM3Gdo6GiJ9tjIrAcsUTlkEaf1hnQktT9MGGPmyCvU9oECoVKE7VyE8klUQwtH8LuB3cp/Rs+sQu1cFnti6Y40lZ/hee57BNTqFTLeOLxpzA6ehjFagV/dtnL0dffi3yRQ9PIC45q3vETTzyBZ595Gu/54AfQmx7G5jundEBX8iWNDNXcqGQK+ZzNOubhVGYpxSgqK16boKgxqxK0WNRUNtM0b2hLr4lC26FuYF3UKLbOHI4/M3dYzpPqcREoisfCstvl2iJmIMojPcyc95g8qmWfaxE3FqO6KowgHcZLr3sR/ur6t+Kay0/C6eddgFC8R1MayKbSQeHUVUqx2XP+Xzau750fqV2PpMPzI7A/sOan4irTaPlTt4O8Fs3gKz/bhOem2xDaNHgqoTlBRIlsB0qFgknOPKWRBueudmWNZrpdLmZyROviuYrVMs9Amy0Spot68eTl/ygY7+/C8t98AWP3/hG7bviUhOPynvDDmIhcq94Io0p0dvkCnHvLv2L/rQ+h+PF/l5skHwQfojG0WmjwwYQ5cc82SzEWIPb3F6LElhRqKAchdLZ1Y/W6U6SxTCTbtFAr1Tz6+hbh3u8fkvsEGUnarLG4alAeUlxk0sSSxVUlFdQWAaMDCRMiELgDTO0Od9AZsmuTzRmpIhGjdJL4bv5E5NUSfY45uR0JCXa7VHuFjcBgabeBLKI8ztu4/s/8mVKtiaCWwN7pvXjVuy7DAzffJx/g933hvWhGK1h3/Hq85JyX4OSTT9Z8XSL3/sXowc1pw78bGlxGOI9Dy1PpNswWZlDO0ySgomvJFwt43TWvxUO37kYwDkSSEURaURwYPYS2bFYHmEdguVa4cf3MIhkpcGJfqaxaX1lZk1pic7rgywM//C8jJn+n7oNvB2p2kaXUtnkt+2HGxAjY0c5h6GYazx6hGG0uvfZsNNswFvG1sUI1RIMkamHgnL9Yjb+4/m34zHsvxaKVZ6IepDA9NeUAR9u4foC6aLn/y8Y9OgL7++5/99Eb2m9cHlgqMXj9AL720434Y24QEwViDTWENnSvD7hYSMNTTUKrlFodcaF2lk54l3XeALoh8KbJPqMVCBVVGu34lJ5v6rWJfuSmasBICIX1S7Hi5n/Aczd+Hodu+TXyTdZIDeRCdfSduRb1YwZQ6+7A488+g4995gvY/a1fIvjOb1AVS8Z8/MyTwOSE9Le1ifI6JTR4KvyBl6EQM08rpn46rYMYCvkiDk1MIZuK4uVXvgm18Qx2PEI9px1EPIHN59ec9326It6sSBhmcs62j48MjOp+M9shZK6MjIRcpNygpBiydh0c7AOtVkj+kEWN7HCNtxximeKmETACcWAZWxeK6AS6KN+LeajyiIsgf54G5PVGAuNTo7jk7efgnlseIrUNn/n+J1Co0eOZEc0irmcrEcEmJ3jJ0iVYuHARli9bhsULF6BaLQlA7O/tRyrbrnp/cuIQanXWcFAv94Tlp+Cem59BiCNA3QAvZmjjY5OqBz2SzoyIf9dBzpTWfXylxUqpbRN6Cx4PXGktsiSRQZo1ctm+4cNXhBb32owN+bM8ZEkHnNMtN41ooXZT3AlmJK90UdNlhp5Qw94+sZZWDDj9qlX47V0/x0vWZDCw7Cz16GlGJyKEk/ERSfb8ZIa8uZcfseMMAvzX5+t0j96oL7Rx+TZJSr8QxbPbD+PLv9qHg6UU8jVzRVHb8I+dJwRMdRX2nfu+indnpanUSu/uepmIIJPNGlDA044pjecoz/NAtjEgNj6YPTW9PxUiyRjav3gjMievw8NnvgWPlHZiwaWnIL16BPlwHcVcXS4Df/6612Pff9yN2uf+U35INqjKUqRQJCTnQHF3xY6x/IDyLk4wr73ueNSWdYKGKV6Zw0lqXALcSATCzv+za3H3Tw8gyMclVayWbVwJf4f5TBs1T3B8rarygWkw02PtAvV0G+q/8iESoCIyLKoneboBLWksarK9RNUKwaVyqaJoEwoZ19lHEppwC+yS2VxNhAfxo5kFxNkHroi6d2Riu/GfmU6VK1Xkck1Um02cdtVabNu0HcXDOdz6wI+Rr+VQKZeM3FAqKWJUa7w2ShkbqDWcOL7JSGtYBqmHf3nD27Dm+HW4+977VAotPfYY/e41x6/GjgcmUdlPIs6RXj5XSblECx8TSIgHnEza3x1ZXlMYnTCeRAulwSIYmK2PbWKTryl1pl0OBRoaMm1kH2mUE2wT2SHEDIxAIidDSPDh3Vy43pzxAIejKdWUHJCoNYOSbXrNIpYIhusqitXnD6N9aQaNyWfQ1rcMM7PUWFuGoo2rWUMmO7RQcaTv4109ZBTgkGGTeBpngRf4pxDmuU3OSEvmYTyKJ3fN4gu37sXBSgwtMtmcvluQ8PaFZwWMND6q+NrBi9z5ht7T2Gh3JiDgQiUB2tP0vCujTjFnJcn3ogiBvFoxkfhQIiGMpcM47tF/x6Z//B5a/U3kO6pItqLIizAODCxchf7+lRg97+0oRo1iGW858MrdFCmSeFNIkVTeaF5SzWYY+XOHUDttRHVdXIO9OHzZmvH8fyiUwDkXvwl33rwPKQTIF4l90EW/rtYF6zRuRn9PRHiI2Exg1V8y8HKDoV3tleXh1zCvLhFTGk2UikWBeb29PYoYrOt40wnvc96Q0mKJ1MMInCkY0de2bHqu9mUNyujMdJuR0JcgfjI8a+RymbOKmogk4lh85iDqrQp2PrkFO2Y2YqY8Nec6yefC66rUawJcKGzIFUwEoXSTwFzdOgepWBRtnV3YuWePWKvMXLhhHnv8Gdx/8xNIVJJoeHsescZ4qIZxaPSwFrgGeCkVNbYcRRfqx8aYFpcRi9hnkRjdWeYSwPOkHgM2LYVmfcznpvqVLUNHVmHtx03d092tDMhHRf4uvg8R7UJxRlGaNa7MDqoVYRlkonET8XdywwUtHrpJBL0VvPQNZ6M8sQHRZI8GmvGpqU3lNq7cT53BocwU3ctvXPVyj+xEy1r9YID5fV+vTXcBT+HRIcy/uHsnbn4iQEnG+mSlMYjYgAAZL2wbeXHg3eOPuOVTQGH8WHvNS0c1IdMkYr4RLsBhvumzZqtyFoy1dhjFuAnsQ4WM/H3Tteh62ZnYeONNKFzcp5lFjN5M+84470o89fpPILNv3JRGfGj6PHZqeU2vlTimnOAG4FZmWlw8phOhN58oK1JuFt5QZhNEYnlyvejsl6JcGMT2PxTN/5h80ybrIjvVuFisbLAHZEJzoKOjXRuP9SgXjBBOhwXIM+lIJiu6H/9dM1c5ST6bUdpGDrT3VmK0tihqtbOJEoBEzJm/sw/sFwWBnWZFogePQPvnUy5xQTY1d7htcRrDJw/juTufRiW7Xy6PRO+pKOLi5rUVCXhUqjqomLlYthVgZnpWYBrTwzotgFjr03OMNXCliVe97rV4yxvejg237tF9YMuDP2eZSRy52YIimqmOSDYxm12+uEnpq81SRBvQtXh4nxhd5C3teq8G2BkPXNarLlJZL5jP1MQwjMw017Nsy4wX5jJAx0BjqcFnxfKEG5iqI6HDySPOjmxTMbKr5xxUcfHfnI1qbidCkTjGxsYUxeNzRg4hOVZKoupagnMbd95UvheqYedHWz9EfW7Xa5hACPFwGN+77Snc9kwUJXCOFdc3cRG2FNxUBQavrSNn6dbyhPSsD90cpgNucpolzs4lj7rGpM1Z8SkB0zVK9bzJHL/XR27eXJmTs8XkjOi44Gb6M1h255fx5Gs+htClAyjEq6iXa4hnO7B2/YXYd8nfafFYP4yxVMN7TT/nUi6lzrx9Gi1CtQijRhOz/XGk30V+KQ8Ja5moppRWs4WXvuqNePiX46iNRWWA3ar7mTVO9+lGPnpvZAm7nY2qiFBCZ+0UjbvBZb5u44LgK5+flSKFBwY/G+1R6FAoET1PcEZS0hmDBhJxo8vxACToVasWHUHAeGWemM90sVIqggB0nGCca6fUG4xGtpFqyQrOuvoMPPZfD6PRvR+hSF2icrW2NPLTDiOPX9Dojv9GJL3WYFupLHF9IV9GKpm2A7FZx8x0Hh/9zKex94kyigfokUUFFrMB6/tycRFDkClIKIR8IW/SPi1u1pwcVGZaaoJ/Att0CDclJ/REFAMIY2JK8XkzQs6NJ5GayGYpMVK3yd6HaqmW2H5ztq1UshWZ4em3S3lktrgGRumQndNEM7BwwqOVNASeTvzzY5HoqKGSm7H+c5j4gqXJfLFuFxg5X1MrEc6RfXIk4DqXEx8C5xE25iv8WFLSNfPff70Bv34mjCJsrcTTZNORLWYZpR8eF9rYc3LA09AMoW0atxA3OeVruzqswT4A00XaWTINlOxOobuFbJL2KO6CONfU1QDeBI4nlOxbHMLXjAJDt34K9VAE93zpn5Bbau917LK16GyNYPz6T6AZNXI6HfbpRuBPLA9iPH/jUulBW506RqNVjHz6KiGkRCzllhCn1I0E+G6ccM6rcdf3n0a4FEFZg7isxmIbQ3QyotsyzQtEVGA08MwZ/hvfkwudJzSjH69JIojACAdMq9mOYOQiP1nc23QCcQIsLomSGUA0JtCKKCgpkh2dBnoFjaqzuXFSSXGlWQ5w1CZnzNuEO3+qRyIJ1BsRFMoVVCJlnH/92bjn+3cjMjCGZst41Hx/z77hVEU9Zc5oKpbVj6a/FFF7L7tT31JZQFP0R0ocb3j33+H+bz+HUDMhk3v2Ejgnie/L665UicQbWMfsoVwqI+nQdT4rblzrf8esNUPVUlsG5ZpxwnkPueG5oNva2sWA8tRTH42pIGrvaDO+tiR7jpghpxRuSOvTckPzuUh258zluL6Zdstt05Vclm14bjTvdxQDZ2Sx7JQFGN21RQe06vK4Hch8sa999MbVWpy3Keei8FEDwPxmt5T3iKVxKBTDfRt24yt3TKPcjCOIJBFTOUXTQmarRGts6IAyjyc7Tgj4ZppNE2f9YD001miG+pl3lOeYdrV3GE3Mp8H+w1Ijqj4oVTd2sZ4RI6GAH1btEDf++8xZK7HiK3+Pu6+4EUuvO0tCx2imE7nxMCbe83lw5LIALtYMtGadP/xXd8YAGlvUNiqF59JMpIWRz74GuSb1oLSBsUHJBHrWvvjlKE6lsfn3OQdImSRLvGOe2hHblKQ5cm4Q74e1dBghOZg6JldFLgJ+tpT4sG6siJvVyo3O+iuRsJaHShlXm8TiVtsxE/HaXKavRHipWJLXstg/bqj2PMCPN7ZWLStdZtS39w6bfVCLA5lt0PXZf/ki/P4/7kHQNqrIrFlznE3sRlkq13QvZlpGBpkHqBCwcUbiPGBKhSLOvOQyFEaTGHsir5q3QsM0URxJj6yq1ODGK+TN5ZKbiuQNuqIoGsq5xMAskUkCAmt2MDPSsW8tRZUiY0htHbqtGLBjBgV8ETnmNbJONiMCo5YqC3LtNJ/t6WASVdM2LJ+HodUWea1OBcLRiLILcYJCYWSHozjpVauxZ9vGudrUYwsqoZy5ok3Pc/fS9+vm7qwLe0fVtM9Ll2WPQ8JTA+OFMt7/9WcwjTY0YmnZvsaTaStnahzknVLGJC44p2Q81XWiM0Q3obv6Zx0dRn9zhm1EgxkxbWK32/FuQfkPwtOUp6IMy3kCayMwzXKsK9/2IJWP/rlM26IxDD/0Zez53I8w/qP/Rq1Vw8hrX4bCypWY/dBXbFzHESbY8yKubrxQYEvNvCkbb2YhEmDBh16J8SS9mDlBwMjvTCXPufw63HXzZgTTxkGm7pSfm6AUr52pNFMjfj91yjwRGAUZOVWXiLFF83i2j5pIa7KCcZe5CZi+8cAiwkzrVxMb2CEoml7UDjQtGNIDqUHVbCACfexvhpFgy0N1HdNJ+zPbavx3Rnv2q9lOESOI1y7taBLleoB6pYYX33g6fvuT2xFvnxQophaPi/TKkhzZRC09j37O+R3bBvYHN593pqcPp5/zMjz2090ojfMwS2rDMjctFug6QbUUyRpGCzWBe0g4yMThMRC447rm16391ZKUL58v6B5ZKm12M6xV+Tv5M1QCMRvgvWPKOtA/oFRZ6bHsd6lAMvDR9RVMyOEGirFNVMznRBflIVcu0zzO+uG85zyQxZVWORZGPEWqaAiteBHnv/VM7N35lK7DJKVO/0uket7oy/llpGM8Wp463+rC39v/8XWKM0KoBjV86N/uw9ZiP0LRhCyBSBhiek5ar9cQM4Mayi8AACAASURBVHD4/n7o8bbj3dawMYEecu8d6AOn2NFipCWWiKUTNr3MwJP5LA/Pu+SHZiriN7hpR63Z7Qd8MdqwtmLU7vmPD6KeTmP3pe9CuVZE6sozkDjxJBz84JcYQp8XZeenygIH3M2xtMXqRG6uYqiF2DUnAauHEYmF0ag1JIfqX3wshpedgSd+fACVotVdOmxicbUU+F9+RhqU8XSjAIK1kjX8WYvGEecM4ahNQVdLQYivqYh4f7gQWA8z/ybwwtm1mjQrX2PycMNSCvH3UnjPeyiuc5P6XLaEmggHpmG1iGoRhx+CRAmZYmtUhqWkXLg8kCKRpAzDOe7mhNevxR2/vAPDi8M4dOggkhzWrXLAMhih2O6/RsQ3FFbAm1hJtBgy2ilbOC+5/Br88ZcbkKkM4sCBQ2g1w2hv78DefYY4c/FyNhDbJpp84eieau3EEyLaGE/btMncJnK6cACWrF8jvNcFpBJsz9nmdbOrVfszI1HpIVDpyNgSUj0ZIFLCFpyxvxu0RrklLXA9+433T6YG6qNz/ZgjBwk/as0RJ6HzZrSC8647DQf2PWMjXnTY2cYV8eN5UfVIXfv/eePyXYMWfnH/JvzwwQaq4QSiqR5UmUlyJAoZhRHXVmU22QwELioDfaxjrVJlnbIOWPC6UD5cwuWkM1LELP4ua0K3YTwyxp8X7d59nYIFRh72Dr1PkC1A9z38PhEammicuwpL/u0juP/E1yA8PYP0Jacifcm52P6OTyFBL2JWdPOr+KNSETvdDF22YhySHx5a2YYlbz5P/s+ZNDWsJZxz+TV4/M5DKOyIiNHj60RNkBdgI4K247Ia+ql6goAK5XrqmyaRlIuE/TsF1lwwMioLM12kqZqRBIRiFktO0sfNwe9rU8bBk7PWrGGQ/Vqi8qRxOiYQf5cxpgi6HfldHVk7OOXCILsX6wmrhaLISxQ6jBUvX4oHHn8M0ehhbRIt+LR5J/u02DOUGHXmUNu6SRB5bcl4Gs2ghjMuvgxTO8vIbyG63kJxhuBVXiwpjprMF8qoVQmaMOMwcYGuwx0MJP9zo9EZhP1gblBD43nomEujPzQUTWS1aoZwJflzWUTm/3VfWTK5mUMei2C05+EkVRVxAL2HqYy4BvnyrC2NQdGAbluLyniSJlAnZkGhCbW/p752Ncan96NSG0cmQ8TbXprV67IXre0/6Xrxv6fKvE/8/X/9z/dgMjKCZrwDkWQbYikzDPC8eR0YPBQ5z6vsNOKPd/iIy2fmhNw6fY1Lyovv6+5BoViw2oSppXcnEDrqDMtdW0ZjMmUGzlMsKtXR3CnvLt4saQI0edGpOIbv/Fds+dx3Ubz5NjRWLkD7e6/F1jd/CMkghBjra3kWz+uXebraUTWv5ztXwsD+jhqOed8VCBJhJIMoIp1dOPn0V+DJ2yaRHy2iWm0iN5szBNNZXwpwopF7vaE2BFsE8xk87GfrnrA/rAFeBHNo5Ba3dNctBuMTOyvSRl1ZC9s+BFvk1FGyOpAiek5akPqFcj5FWRN80J2SiziRosVOzSRt/JqrRTV9SYveAT5kXcFqxkUvGcFMq4idW+7X93PR0ZXCz/eZnx7z+0WcbzblgMHPxgxgejaHk847D6F6Gvv/MIFIPSHTuVYthG3bdittbYU4gnQXopGEEHxrCxGoi9mfmeaqN0y9ctLRLW0DMt0XAUL6VcMMZLimdLklVNk2vVFRBeD5WtlpWg1INEsfIueWNFgLju8ld01xvK1lqM3A9l7NLHI8QhuX8ZuNFCEQ19HWg0Uv7kX7ghRmcns1cdIfEqZimseWcp9Fh59b38+PyPbF+dkp/+4Pt3/+3u/w0P5O1OMdCGe6EEtl5iZ88B1Z2xPxVgChgUOFf28h9Ejb6sDXUX7jGo/TtTvicaGfczYf9L2RiMAr+e1jegIGHwSlbGYcHAicmGs/zAOoGEWJTIrc/433IGhPYsuV78Z0q4Ghb30Qm1/3fqTnNi51u4xiBkZoRIpP1d1dkvLPAQTVoIWpZB0LPvpq1Dl1oQJc8qa34rHf70NuWwSVnOmCebLu3LVThT+nnIvW6HymvDO9IZRUBxlARy4uox2vV6AK7T7TSUOsUwkdxroHHIfpwA5mLGQv8exhROSIjwUjI4rKjIZKT1kvp5lq07mBdTEPPJYTbIdERCAgiOFVWWzHqD+udkkY8XQalQp7vTUMnDSEjmP68Mh9P7FIQ9Sb7RWX9YjcMEdpZWpL8zue8lb/cqEsWbUG/YvW4sDt21GpxFDImWEdSRbbtuxCe0eHShOiypOTMwIAdUjI8tV6+Hz+smGlY4WqbE9RJJLvNhR7Ww4f4PuzfGCqPDw0JE41gSebD2TPXGmrR9ndIC0Dy1ivRtDRYS0i9qNVwpDdRkxBLUT7/VxG1YoRghTN5VkFHTSck8T+P4arOOeqc7Bj15M24REUY3BihVbakbxv3sb1KPH8+bj+G5+/ce2zTE7n8defvRulbC+iySHEO3oQTqTkq+XZWsQseD28JyySWDaICPpY+1pRoYSMuk3ATcpThjeSi4kDovUglJPbtxmiduSliepO4cHL8ubbjFKsaZliqLZxvUfJ+Pyg31ecjp4Pvhlbz34rytN5xL/0Djx04ycxVA+QDMJymHy+K8SR3+3TPP9J9LCCAGORBvrf83IUExFc+sYbsWdzGeV9wPjeaZRmK4riTDX52fI5yt2sXzjf8Iv9OuPb1sQlNufAqA4RXn+jWlebhwuMt49kACO/N5Ei4YLvx1kvmixvaHKj2kBnZ7tmACnFdQtSelJuQIrtOTLDeQlzCh+7SBwh4iWbirp8RhRjiBLJGpqzY81Ct2tJB5acuxz33v4ztLdnMDY+qgXPQ0GIrwO1rN6k+39R94F1KOvyxWuPx4LFq7Htrl2IluOoV62VNDtDA3Nayc6qFqQgpFLiPNy8XE7URZiHgTDWx2XH49a72kQlJFPcyA6s0wRHZiFFHXgExej04QeS0xHD/L8ccUezhoydxmyF7SYjuqS12AlAGYWXkk6T+lk5ZWNMxCngoPZy3oz2SfaAlYTm11xGOJpANZHDy996MXbu24QIsQcX/US6cIezJknOYz/N7YZ5GamPrnPMKR7dQQQ1FPH+z96CHaXFaKQ7kWrrRiKTpZWh8ebFt7Y51fy83LBSvIt33kLo0bY1AReAPoAmk5nxFT8db4D6qM7sjQuGkUX1kRM4z31YZ6XJn+F8VR8RWf36ekfpgbtQcoz5+/igC11JLL//G/jjyW9BtJxD+IPX4OEf/QLdG3chQ1mRU8b4lMPD/fNTEJ+O8waRZjlD5PDqM3HBh/8WhcMRjG2tojLZwNRYDqV8WVRJ/n5DM9lTY9O+qEXNjapF5IyxCckTxWUNZKQLDgbjTB2SPuhRZaATWxncAOIic8GyHUGgq16FbFZLrHfTKBbzyGTpF30kjWMPkveG70WKKP/Mz9Pf34NKuYAoxeHsSTtpmmHJHnCiEiYudlS2pxvVSBVrL1+Lu371X2gFRW1wwzCIskfmNq5q2WTWMopwBFXW4/1DOP3sl2HTHc8iXWhHhZMWNfeX0+Zz+r6JiRkd7FR9FQrcPBmMTdA10iOwbuCb0n5D7bmB1FJEQ77RJPHMIa+thq6V6DyRaNXicqkwxp0FFjusxQtw3lwUshcLeSxZskQOHbn8rNJrk05yE9YklhH45gCtufQcRkll1pRMpw055gFCgCybQTKdwLpXrEQtWUJuclxRzrO45rfT5kfU+evyhTa0slRRJFvYO1HEez/3e+RTvYi0DyLe3ql7yhGyxEq4z3h4kdg0V5p6A0K2g7Rx5/UhFcHCIWRSWecAAelpmRtKl8qr89P0XJTWLRU5w/yAaChmG5eGcZY2zQey3BGoTaCaJhxC/+PfxrPv+ypCv38Q1QtPRLBgEDs//210BMa+YVrpU/T5ULscMlzNoNRHtUqA0fY0rnz4R5gd48jIJqpTZRTzDVQKNREt1CYi4lksoFY1hJu12dT0jOor1U6OTEHqHxegro3v3wo0c4c3lRan/ABsu5ClxZ9tb8/KwzebSqPM6X01MxqjQKEldhI5zDVkM6aCUZSNmhOEDkeqfep1ETJo2VKv0nM4g0hg/VF7mWeT6JMNglQsTyJo6+1BEAuw6IIleOD3t6NQ2Kvszpz3HVVQLRhLr8jt5ufN53JoBlG89MqrsfvRPQgOhjXcKyAWI+8t/r4wxsYPC9hjxC2WCxJ412stkNQhOicJDorkloILMkuQfEJDd0YOpsI1lUk84HhPNc5FKbbp0KSskh1QXFHUDhbbuEqXiTxLFM9B3swSOJmPkZTCBJI76PJovWndI9fnV8bnhpyTK82+uRhbLtXUNQZN9A72IhXN4GB4B172hguxY8dmtBzpQp/BaafnJZxzSL3/2p/auBHSGMMVvOPDP8b+6hCa9NNuX8j+lAbhRTkyJWjo+UsUYnwoHboq4R3fPPTH7vU2rc/3TENAxk2Q583wqiBvVmBpsOtpsYaRhzKRX9azCVQd2VunrzyUjzT2+TVvS6NI7m1IEKDntn/C7L5RTNzwj5g5pgMj734z7r/qnWgTTzo8x31W9J6nyODpJ80sca5mCJF4EqUVwzjz11/FzLZZjG2rojhdQatCTjLmVEBs4NuDYl1IrS3TVqKGxtFmCspNw542U2qe7qxPeRdZs1k5HUYg72SysxpAqIae3m7r04aZ7jRRnM2jUa3pfYylY4boXNyVUh4dnR2OWM8WEAEu1q0G5hABZcRhFGcqVy1NC+Biaklmm998rMslzaRRWob0wRgGTxnC/smD2L3lXsR4T0oF0fz0DIRZmFhE7k9BIMLDqRdcgsl9VcxunEWrGUWjbtkXgSd+D+8Jx2hOTZLOmEalYdI5sqyYqXhnR16bZ+MxSjEFZ9sm7GprRdGgrpqfhndsLdFjir+D2YznePv2ju/zsg7394UKNQKWTCWJzAqoi1prrZgnSYTtS5YxBMmsDWb9X6uVNamwRc6xMayYXbFXnMok0dPXp2wzlIwhtSyEodX92P3cs3P7lHdlPt1RmZ+TnM7fzD4jnL+ZqRLPlRt404duRS3eA3QNIdnVg1DELHk1b5qqrXIVFWpxnTrPPMiNjCRA74mudQFbPV5/amSAiJBQf8IJineWH1IJemDDzWxlOpJmisOer+PB+hPHD13yOb5aTc7RXmCJJHlNRD/yJvS84hxsPfU6zCYaiH36emy89kNoZ/3BZhPbDO4OzHfNI9fYUENu8Dj63/QqLP/oDRj940HMHGihNhMgny+JylatmBsDwThGByMNkAVNdJgLs67emYjqqseddIw31AEDAnpkpm10vHTMFod6oFHjMGeyaU2J54FWzOWRcgQNtUGcn5babBznQXJHMinU2ZBGigxicswgiKWSLmILktTPUiWPVMKQZ1uMRkLhwoln0sj29yGZaUMuMYv+lSPY8OCdKBbH0Qz53nDY+pVCV9kXjqKrqw+9CxdjyYqTsfv2XWiWIqg2WC4YEBONxJUm+tJm755RFIs1AWIqNajGd3Wn6WTtsOZPa+qiy6zI4ZKsjiUH6+NqUbUpD1HyibWhdIBSxGLiDF8CMZVmr5UgV1+fs/LhweOnHaCltptlFWzVmeWrMees9UPChge4uI6Z+VCEQracX/8dnW3ydeYG6h4YQD40gzXnL8Xk7CgK+cIc3/7/tkGP/rf5GSIPi4/+8y+x8XAK9WQPIv1LkcykEAlbf5sBgPpgkZ44MJ3llLMx9k4hyoofyq4ShMyaw99Unpysz+RqSEcEWY2YKsdL/GxhM4Pmmc3hTil9wdtk2oNjjLf+rU9plULzEHCT+PRQww1UXnseFr7rWmw++TpUQhXkPvQa7P7YN9Cey6MrnJS21r/mQBqCBOoXEqKOY/1Nf4vsay/B3sf3ojya4GhTFKermnvKVJAkAfZR9dlbgU1g1xhMmyJYoZdVJGY6Wk0WbJlxma7bXAVlqeMWgozO6GZYMmolPaVYLDdaDSTTUd2PGGvuitVpOvwcOV2gX5MAldH9eAncHOSB9/Z029eUHpqti6w6xVclH7hoKiHH8GKKzjIm3dmOZFc3IskUplqTWH/Zi3HPz25FMxhFHeYVrc3EfrUDClMZaqtDuOBVV+K5329FZDYjsnyrboohEVuoruKCcnYt+/eNoVZpIXC8YJYUHELNtJb9XRJY2BbiRbOG5DPnPeW0Pt4n8pmjHGdDQbyTQpoai5pgI2NISJBg5DYLVqbevF4OaWPrTAIQaZ15z00QQw6zhAt0Z9H9s/6nJ7wwhbbpBWZFxI3MDS4mnzNnZ4eAJ0b/YD8yvR3ItrdjOnQIa89dhmc3bTK85ihgdn5Enb9Jj3z9SHmTL5bxtg//GuVIFxrt3Yhr4yYRallbj59NGAvLDreRVWaaBGpOlRb6Q/a4INwMxHAhsVtjDtwbWI/NHDD8KardzsqFUdgJ23lj2K8VgVxjJU1+NHcRrhnvEWBGT5uT6njGYaD4kuNwzD++BxvOeBsirQam3/NK7PjBr5B+bqeIGElK4o8iYjDZI8OnFo7good/jOnuXow9th+NQ6y/6qiWKJCvKYKZyDqEsbEJRa9MOotcPj/3wLiwGFIqdSpSDBDwNa2RFdiftHTQj4vkwZRxSKoiIiN5g86FIRQqeWRSSU0baDW4cAsiVGh4meprHoYG8vFwjEu5VENXV4csVxhdpL7yWYbIB25iBA3Q6JkrMQhTRANguob65bEc72hDvlnB6kvXY+NtT2K29hRKTdO+MrJwceZzeRNJhBN48aWXYXpvE9UdVQTNxBwrjNnXxMQEUumskUTC5B/PYuzwLGZmiA6b+6OymCjdUdiSMqSejDMePJRCclPQ7jYSbpj3kxsKRyIE570QFGP7i71vWcs6yx4Oqg61YqiRvNHeISdPKqlIE7RgYmUSnxXpq+0d7Sa0JzPKbQCapPMmcrPz655oowO71ZS5O1Vb/LuZEpSwZOlSSnWQ6uhCRz9/bx1d6yJIdWawc9s2M2dwr/nkIGPwuTrd1aN8fja0PYZGqIgf3vIAfnrfNFqJbqB/EVLd/WrFeYop12mZg+LqbJkRvTVWm2+1WXkUIHR/emVAhDTLiMkERpvP0dJc7UtChbXx3UtpGsGKQBFCFDU5CtjPqz/riezzkGRFXg/Pe8E9iRocYbl8GMM//gSeeek7kZ7OI3fNOXh28yZEf/MQkty41CTOO+l4AfT7zQ8P4OX3fg+VYgj7Nk6iORtFpWhuG6V8UXUaWU2cK0qQibYoBw4cUF0Vo4Y0n3N0RAOomkEIuTxTKBNu8/uJ9Eqe6MoA7h9S74g2p2nQzUhCgCkW0UR2kQUoJ1R0toOPQAgb/7EwXS+Y1vMmEtU1twdyFbt7ekVW4Mb21EDWfOLSSs3N1LAJpZxBzTjBXIAuemZ7OpFqzyLd04uZWhHHvXw1Nv12B3YfvgfhjPVVjW5qjDA+i1K+hD+77u147padCNdZY7PGZAlhdZw43rwCN1FgapKSvxomxvOIOg8ylVQsr9wi05S5OMdC5uSzxfvOdg9TwGQyjmicQ62LaO+JINsRR7wjBLb+YwkbyOXBrWqJnOwQ8lNljO8sIKjE0ZHtEoLPZ8MsTx5ebl3E4sYnlxJKHHlnbyNKI0UiVuMqnachBANGMT+nhOOa4ubPtmUR5yjObArJ9iw62zqwv7ATJ1+4FvtG96FW4oxae70Qq0+HrV+rag2xjRpDNWjgmnd+C7nwIKJdi5AYWoBwOmsB0GU0co7kYcyfbzAzkPRBb2dSTPtz6IHscUFc7o5E6szIWoOU1OwmeZ6nnvOfFVDBm2FvQhTZ80WYemiPUq6mVMcTrT04xVPyyER6r93VCcULWzSIgdv/BU9e8T50Pr0XB4fbUb7qRdj7ia+jB3EkXQtANiNKm0KIrT4WZ932PUwcmsL45gaCfBPl2QIKlQC1EoEd1l8t0TW5mJg+8b/9/f3Yv3+/wCC2BKjh9QcNPYRmczZwWYR1Z9BNhNTYYIZa8qWay5P9pQnmQC/WYmHQrpbkCD4QuTbWyygUaPNZ0MZRKhgmAk35Wgr93YP6XUoJo9bP5f3V/ReHmMWujafsaqerZkk6WRrmqSInMb+nC+muNqS6ejFZnMGqy1Zj6x2j2Hv4IbSSs4rMSiFpuCePYfkE4pVvvAEbfrgD0RBrSBJcmMITLDGmGK1x1Gar1zE6SmF5HHkSMlxfWCm02xCGYVgLkJuQBxZ/doajRUJVdPSEcPJpK1FJHha6ykgd1JnCsuZnVmStOLskO5RIl6zWSggV4sjtD9CcjSPCodk6LA2TMRqkyfr4u3mdbKsxS+Kf5UDikHhGZ6EWnK5YKQv152Zgq4n3PNOWVV86mY0h0zOIbNaR/kca6Fnajp2bDagSc3deFjg/w5y/cWkvzOf0wB934rPffhiNRA/ifcuRHBxBjPOZKXap1hR1fe+WtbtIR9q4NvpGskQCoXzuj7avkVmcB0Y09pD/88Zc3MBC4MypkOCTX9BJkbINJZ1Le90i8uGdC1hfcj1Hf1IJn3Xu7GFuhs4khv7wTTz7l19A4vd/RK09jpn3X46n3vFxLAyldcqKG8rFhhbazj8DZ9z8BRx8egwz2zn2gkSHGiqFskgObF2w1tKUPFqQcpaNc+XgZzAksSUHP8q0eFp7WRcjhTX46WVsKhf2CT0QRP6sjdZk7WtqE25GpuIkSgTNKtCsYHziIA6P7UGrSVqj8Y45aEwAl0tvfUrOKMrabu2q1Wgj9Y0T72KMTsyE3Oneagjt5M8kOduoMEOSI6wCJEDZj0gmgUxnP6ZLU1j1yrV47rY9KNXHsO3QHxRJGPHiSeqAC+aK2DaIc/7s1dj0o902uM1EgIhFDeXkM5+cnhJnmKf9nl0HEQRR1fUc68Lv8SojXwpR2ULQJxRuoZDLo9IoAdESzrp0MULxCkplTp8iDdR5kSkS2ybTjB+3YjSF0bVodM81qK1FwB6TW8qY3E2ZZVqZUyxpkxRMKBHRKBJbm6wbmyIwZNNJJ6yvzE1SUKrfqAgk0+cPWujs7taG5AbOdLQj2dmGTCqB8doMjjt7IZ579hmNnqFAgPZItomPjI19XmboWqHEC97+ke9hX6EDQXYAyZ5FSPQPWztP9jQ2zbBJphRH68kS2Ea3KrJz/zmaqOZXsR1kIdhefuMaN9hFUaalHIdAXqy4x4Ta06hpSp27za6O9Tm+P32YJvq2j1hNDlnVUe+yb6J6QTqKkYe/i22fuxn43h1oRAIU3nkp7rvpC1gUTyJFCy1ukgBof+mZOONHn8eWJ/ZgZnMIyHMKm03N0wgWWo06ckc6lTErFkYFprqMUAJ7rN/IBzo9M6u0j0R9LhS5J4gDTEvVrDY9oTZTvxiSy0WnVlmIJQIwPT0htLRWmcGh0e2oVui95LW6jkTChe7wAuPz2n2XKknjWCxapBMJ9HR0YXhgELFIco622Nne7iRm9pQ4lDpUr6LJD9BsoWfBEOIEOtJZlFHGsouPx7Zf7UEQrmDz4TvcLFoqT0Jq+fF6lq04ESPL1uPZn+zQac5+bCQes7k/DsvgY+JG172aLiJoRjE9My0JGg8btnr881YrTBGdhJUois0pLF2TwfAxMc3z5UahAGV2pqCNSnosQTmLKMYFsJ1gA+CYYfH9GX0kDuB8JqWTAcLVAPs2ziJR7UciltIJyufFSMu0XVkUsQoZHJCBZsoqK/NsM7PmJ/PMwDSzE+7o7tThlU6l0N7TrZSZh108nUF8pIH24Qx2bNtCtficc+XcBvKbeN4XeKgWKlW89m/+E610F0Idi9A2tBiRjB3CygxbTdkJMftgYOLn8BvX6lsCwQZe6faQq+zLUAJGXLB82QLz99CRLxh9CdK4ERGs0bRx/ffN5w97JZDoeTbvVfWFK+C5AX1KxHQp2p5G3wPfxN5v/BzVL94ix4vZl6/HQw/ei+HRKYFT5PDGertx0dO3Ye+zh3DgAQ6RLsn9QRPxOHCMzm9y5LNeq6HFjIaOteX+K3MA+hvXaihQuscSAUynTaxsfWabycpFxZRKG52nvqNqEgCxYV4VFArTGJvcjlxuDNFoSbUsDztzEfRAHVHmhA4Wk8+ZWJ7fx9Tf92WZsnGLE7Q5cc16dLZ3akGypJnjG3OiTSyCSiEn21ue0D0jQ4gmE8j29qIYKmHx+Wvx3M93Ip2O49GdP3KsI0r1HJMpaOHMcy5Ftd6OQ/dMqHXDe0ItrMBHaYCr+p1cXASYcrkKWk2OSikgqhLESP1il7l5wXx/orV9I0n0rS6jgSI48jrOrENItKWEPH4YSTWyhemiq+FMRWZtMHlVsf1IYwORNzjIyonvqWEsAwefmUayMoz2bLvUXRp/wllURLSdeICfrVLMI8t+OAUJ1G0X8m58qm1c/wwSqaTKF9a7HD+aaMugb3gQyXQbirEpLFzfh63btiFoENC0XNmDt3PRd97GpQ/yb+7agH+9dRciqXbEB1Yh0z+MkMa2WgYrT2sGQpJeqBSThxZXvG1UlbH+0OFvZTvI/1IPHPmNqwPI1Vi+t0nXRAIc6q85frLjSgoplkcuh/w5SF/hqNFU2id82zevmQp4PW2oiURPL3oe+Bq2f/6HCH3ndpHQ92YD5M9YhsKtv0M2mkAmlMBFj/wE5e5hPPGzLajnaa5dUCQ1T+SQasbZmVn93YvGreHvMwNbENq4nMlKI+1GQ/pgO+VN86g00bHImKKz7ufi1YPhYGMuxXACjWYVk9NPY+GiCvbtGsXE5AxCQVI/y2nsJHZQKKD3axmaHo8yRbQ+qWxjqVt1Nj38rASkGOXVKmsEOH7ZSiweWYQ0hQCKGrZYWKuaTM1cR9p7u0V5pMKkGqth6QUnYNOtO1VH7pq5DQ06BfIwSiScD1OAi175emx+chTl7UzVLavhYiLoM3/zkp9D5PHRVAAAIABJREFUp4tcvozpmYLmB0UTJikUGUGWrNaLrdfLGDwmgcXHN1DWfbU+Kj8r2WNjhw/bHF5NKgirPqbeli/2a/nypQzfmwyzYjGnTcwoqbajyjP6UYeQL06hsD2EcKFPw9nZzlLa67jEnhxRyuc0nEwRu1EXXTKdsdGnxFlY5tS5bqIxOW0wE+jq7UE8k0I004FkNoV0RxI9x0Yx1SphanTP/x5xRROu4/K3/Qtq6aVItfUjGFyJNg6n1oFYM3koe7bMwOTNZg40Kj/dxtWh7sBiZbX3pldwjTk5mZ8DyzEVBjSJ5jh34+tIsX5xUZmb0TNSlKI69UlEnEurYUXgTiT1gVpMK72W11EndVqFm4iuWobBX/4znv2LTwH3PcUGHKZTLTSuvxjPfeZrGEAaS//i1Vj7ib/Dk7dtRTCW0DhGtgE98drX2uS8au4YUVPnhC/k1dXjBKV4itPxr8wp8tU6pmdmdMKSlEEiBvusTBvVxxRbxaKELTQ+3Aha9SriqZ1YsaaKeKgs6h37wKGA9izk+LaQmy0hXwyjVGggN0NeM5HmrJwWuAClG43aOErdC01+sPmxjBocaBbUW1i3fDWWjyxR+nZk0XOBh1Auzmozd/b3ItPdhRBTxUQDx1y43m3cKLaP/xahFIeQtaHWIEhnM3hect4VeO7RA2jujaDJFoizH6J4wlM+2XfloUX/KY7YlKkc6/95jCRiEDxsuB76FkcwuLLGjrMOAx70Skk1k7Y213vl/UxzfKfAIS/xc5xkN8VQ3YNoTBY86hfX6PVF0X1Rm61RrqERaaKVr2F8WxmpSj/SiXYdJH4kjieAsF7kpA4uPTL8GPm5cYlTELASPiFyjQFz6jzEY4hlUkhmOhGKhdHe3YtwZx4DJyzBto1PooEjE+xfqIfLzz86lsd1H/4ZWul+pDv60eo7Fl19vXNBguWD8AWJC1gyEFU2uazfuPwzywWBpAQA78uulJ28UkOnqVV6Ic8hywS0eF2Pljas6sM6cMk0kVxczieJKhcOfXL0LEYTpteqsWWK5rpg82xpIpEWkte+Ah0fuR5bTrsBsckZ2ZYcStTQ9o4r8PSnv4W2/n5c9eB/YirfwrbfjKFUrDvU1lJu/39t4oYhyXxgU5OTc5pbXrCoi06ozfEOpUpF/5eLgxBiM8uWVlOEdZvDyptpaDqtJAJUC3n0DBzE4iWHETTZNqmiPduN2Rxnu9L6xc+9iciZQumO0iCgVongyae24YktE+hsa8dLTlyNZokzm2i6xkyag5pJajBTOKLe0SCMM9Ycj4V9i0w8r/voiKxNa+/0DPQi2dWJVjSO1EAWg2eswDP/tVXSuP2FB5FvHNbnIPGgs7NLm/HMc67Apkf3IThI5NSyFAlF3JgSHrTcdIVCWQdaqVzTxuXfE1kDznjYJZIRTZUbGGlH/6pZBGSOEbRzNjOkKNKOtlgqOWNyox1y7dAi1jIih54T4XXmdj4bJGupq6vXlVvUKhtphob/nH/M2c5BuYXn7plAX2IREsk04gn1H8xtRAcmMDs95TjMpgcmWMcNzWyBXtcCKmNUxaXNtYMlA3vA2XYh1vE0dbMVLH/pWmx9+hm0wjalns4f86eRKKMTs7CFH/33g7j5rr2IJPsQ6xpEZuEKRElEqVudTR67zBVZvzpCkApW9YCspFBP33GWVXrdk12hjWtOFRSJ/x+q3gPMrqu6Hl/39f5m3vTRSBo1ywXZwtjGTVRjU0LiNIwJoYQQev0IBPhB4pAAST4IhCRAICEGG+OAMTYG3LtwwZZlW12W1aWRps+83u7/W2ufM9J/SD5Lo5n37rv3nH32XnvttawuYA3qT1pfixKV5cnqeZpsAfFLBAUCGX70jyAP0y0BWnEBWiJza7jawAcV2g4Uy+Qy6PvJlxA95wzsO/c96NRrKHebmE220HzF2Xj8jofwzs99Hqs+/Pu494YtyNX7MDs7pw+biLnUx2kVMT3Se1OKRKLYRn7n5vMsMNZJfAisfSkOzrqWI3yk+Rlf2EV/vpajPXo2D0+JRm0RgwOzGF9zXAymUqlPXrOdjk1+kDRP1Jd9S35e0tZMo7gpggGnkaq1Lr76P7fLKPwL73kjwghPd05MBRpW57V+/8e/QaXDnzcw7LLz1uOVZ12OgfQqaRTziymjSc+GIm+k+0uIZ3JIjuTQf8F67PjZDkXo/TObUQmPazGTkNKhtWqng0tfcw32PnMCtQP0ljWmE+vpxWpZ78kFz40eCeKYmpxVKsnsl6OQQeKUAiiJGcm+EGs3NrH2jHORTvVgenIOM9PWDuLaq5TLOn0LhTwGBtNohgsoV2cwuzCrYQRpKVMhgzy5bohMIq9WDlUvyN6SxxXLB9jAvjIWyQpZfcxUONpI4sAjMxgsrUSUcEKXabOVaKJHkuBQLUuQ3VRKzKmDLadMljW7lUNMlWXyJVO5KFJ5km8515xGN9LES996AXY+fQiRxFEzaydV8zRzavKyaVVCpdA/ec830UivQyw3gMTYOErLlqPO9daoqw2kCTKK2JGYQvqoJl7dUEVomIuxELl5Q2sx3ptbp0F6r92rGOXsG22HGVDlGSB2ctqN0Hcdw8hrTqmWc/Uv0zqefhKdc8HBc3XjolDyRnYQFNNYvvVGnHx6D+p/9i/oBB3Mtqs4HJRR789joieNq/78/TjzbZfh7m9tRzxizBzJvTruLxehGDzauB0QgeVJQRYUjckYnZleefkWP0RAqp4AKfYrG3WlRwYYtKVswd83MXduFPZ7O4iHc1ix5llE0EQ0QdkTU/zgzK6BUVZfhQTMmm2107woPE+raDqOaBjB577xE8SSSfzNu9+IpCiR5nNDKR3K3PzXzQ/iZNnsTshsu+jMcVx+znqMJS9AKk5dq1Ou6gzHHCLPDfUjwtq6P4mxTedh283b1O88PP8kZhp7RSM0CZ60FEAuedU1OLm/hoW9DDIEEdPiSUsxkzTMas3UBVtdTE/Noc2gU29ogJ7WQZzJjSXjuPT1L8OhF4+jPksYihmWTU3RGZDrSzpRBAqlwUzP4yi6USKolA3i4DiF4aLI9sVR6Ith2fgAqpjHwuKsergMoDZ6xwzOQDrvGJmnxGu9hlatgVwhg+fv3QtMZpDL5Di6b0olmkIyjyDOR3uZGxmQU5FycUGzy9zArMN9y04kf6LfuV75KEXjSTSjLVzy5xfj2YePoTA4gw4WbUjFtW6k5qF6NIqp+Rr+/JM/ALJrECn2Iz++FsXSICo10i0bQpLbbI+xdFFj2IzePFCJjuEztq6szmVPOLgnty5coiJSBcBN4jDdtU3vZ0g4V2cu8s4T04mWmdQIh925tOUMHolqlItvQJ6a+LkEMVwqJL6zHNhMiLozWMTIk9dj5ye+iZ5fP6M0bbZdw57OLCbjHWz86/dhaPnZOOOq83D3N7aj2XQ2iWpSGynd6kPjLbMm40YyTSiL0kJK2bedm1OdSAofa7I6c9MuKZI1JNNpjeNR0VHAgUAvOy1JqjCSxjxWLt+FZHIRrWYUuQFOA+WRTGfUP83mehFNZJBO9yr7Y13IMRi6tFcX64ghjliGtWRELCe2ctKdBTQW66g1FlCj189iGeW5OTzy9Db85I57ZF7Nh3nhmWfhsgsGUWyvwmB0tdH+2Hohw0Ynbg9S/b2Ip3KIDHHjvhTP/OgZtUcOzG5GkJmS1jQRWva42dIbHH05BkqrcODRE5qMKZV6dA/lseRmUHkP58sV1KpNVBumQ3zixKRQ+J6+IkZGR9BpdhGViiUXgpOl5TnRNXcBtZpEYjGt4yRdHUSMoLyNjYAyZaSSf5tjXKxDmzU0W1W9ZrY/iUIpg9JwEYt1utVzGiqJeres0oIpIu1EQ2pDLwZ46vbnMZQeRoQqjqfRD2WiJu451TaJ6prtjQbVSUmNccyx4MYKTRObP5BKskWk0I1OsovL330pnvjVIQyt6CJIT9n6s/PMiSMAnWaI791wF25+YBJBbgSx/mXoXbNGrSt2MiSNxIyGpZqo2wTbDFOSzahcPKxzQ5SZ2YLkkZg2/ya7Zmke11tlcjNQVd3zkvnJhXKx9RM3JQZtZweoKBrQfyhktGVLKYZcYMPm/B0Spjkpw8hlBlDOe1cnfQTtP7gMy771Gex52ftQoNdqq4WZTh1PN6YwE29g0yc/jGUbLsbKS1fhl998TqmkSahyTtY2rPVBjXLJZj5JFFww4lG7vi3THqV+buHyz3wYhOHpm0OgiictR/AUDNhCaNYQTSSNjJEJcfErVmLjRSvQbLOma+PAzqOYmSrbYqi2kE1R7yiKsGISI2wruGdvi4Slgzxnjb8svnA0wCInVeJAIhUjrVW2KDz5Vm8cR74/jlvuuBVbH30c73zrJrTngebBBPoLg0orOxq/o0VKEem+HgSJNFKrchi79GXYcv2zmk+eaD6GVnDSdMUEfzHA0cN3A8654GXY9ZvDGgDoKZEKSjc9Iu3W+uKpu0jt5BA4Mb2ogMfxPhp0jwwPq1TyShNauM4ki382BcdT+timEMLRSJOo1dQPMRCJCLS1WHUSaR6Vvd6YNhb1t6xWZX/TCctziAANRBIN5IeyGH/JEJK9EWQzaWx7bCdmtkxLWYLXRsCS7cLFhXkro2j1kiDLy/qlTFs54pchcpzJ6DPJc8qpXcTjedWstVYL+WVZXPSWS/HgzduxfLwH0b6jStm9bKtknniX2028/69/gD3TRQT5fsRH1mBo9Rqx3yQWWG/pXspbOogiSnIJcxAe2Jovpv2qqZ3QOoeaYzLvZqr8y8IaJnYGOBnp1eRZ+IA9nN4JDWRgFKTjHFUfqFPbpfdMW4oTnF2MDfSojxjtzaEQTSI9U0P6yDzyQQyZ0Oh8nJYRYubSbTbc+3/+VUSWj2HqlZ9Eu07fmTbqQRf3Vo/gZLyOc173Rlz+rvdiYMMI7v72riUShyhyTppVrCanC8XZUpLjBbjJb9a0hfiBiWJyQc7PmbcP6WgLC2XUm019Dr4IEWcutlazo9bJ+o0rcOEr12Pn9p0oT7YR1uyz8D6xnrUpIPZR3KA2g0eap7YRWtjvkxwz+7BqrDMTIbhmmQNH+iIa/TObDNZiXMwiM3YB8owi2QbGNyzD6PIUtu16DJV9DfQ0ep1nr0V61qaF/l40IlEsu3gtCmeuxrM3PC/q4Ynm4+jEp0BCCjdmtVpXxJ+e6cNVV/8+nr99vzIgyu+QX8xgJuRW3NgoFqpVIcknpucwMXEC685YJy0yotAqExRALYAQPPNkeNaf/BmpX4hsQH0rcortz7JpbZtesNZFp6PhD9OHMoUSOfYRXHIqFaT8MSgzh0uojWYHB9dUPbKAtRcMoHdlEQ/+zz0oZcfUZ1YJ1+miTMlcotSSCWIJY4rTTJ954kZiEW1czUDnrBwR6huhxnGAMBrFqgvHsebyjbj/hucwtiqD9OgJE7d3Jy7/w4EI+m9d8bb/RCs9jGh+AMnlZ2B0fBUqi2VNSzUrJA41jeevxUv2FGm6DFIdySJHui1RfMlhR9vLP3UR/CK3WuCU1Afk0yrPQWkKS1ep00a920UlaGO2WUMtao6g6jG5FpDVwaxnzDE9xqFrJz/C18h0I0hH4lgWy6IYSyIZOFUL1obpOMa2/xQnvvsrdL95q8TXNHoWAPdWD+FgtIqRM8/FH//Dl5AYyuOB/96j9IqRh5uL1iCGIFvN42VkZeLklPK5eQhQsX7jKcs2kLxuKhW1fCq1hhBlL1zOh8yNhxTw2qsuw/TCNKYOLjDJVeZgGAAtNHgfTLGQIgIqDQJrpnMhSfxM8q4mvcLvg4GuZSNyGgM0QREbCm93kJdReFe1T1xjbUSYOYETWtssE2LVOT1Ysb4f9/74HqzIjZpCIqCZ6Gwhg0RPH0YuW43U6Bieuv5ZpHIJzGIrgtSihvQjEdaslvJue66B93z0A3jy5h1OEzpts8Ed6kIvuuujvUkTEycn8cKBg1i5YqUc8lhSeN66XxPcnDa4buqNavE6FwquBbLYGJj5/IxH3LTZU4eV6BmmUkpdGWDJ95ZAmsdV2I5r2SY2qVQ+AzMm1ymnLKmJVryG5WeMYt+2HcjHU8jSYocGZa0mUlQa0VohN7uDRq2KTIZa14biExPgNTAQcu1Qj4xkmVQui3YnwDmvX4++1Wvw4I+fx/CqNJKDxxCJkmtl+lpm1cryMYZXX/t9hJkCYoUR5FavR09pQCCdKaOw5SeKn+mVc+M252XIztOWtX/A8kLpLenGxD4I7gYIbi2sNQKGEdzEveTGSQdxVBp1nIw2MUPurWmfIqmFazrKS9QqH2nc3KoYGC4lJkZtNa21g3JNYFVhAL2kqEUjSF16NoZ/+E/YecF7UVqwi+XTboQdPFQ/jF1hGcNr1uOaf/4yOuk0nrzloBucj6lWJW1Pin6sq2NuAH1m1lJXV/96aRJ+wkq1opOWNR75rVTTr1IeRsyVhtQQudHGx1cglyfnloPzMRmDeWCNlpj8ko4SaXpk/lDGhkqGFDjPZMXSkayqZFFtgJs1HE87vo6EzCUI7mw2Q0OOBYRJQTIuphI/n5/AIkKpzglqaIV1XPGnL8Hdt9yJlclRbf54NonSYB/i2SLGXn0m2ukinrphO4r9GXQKL6IRmTUiP/2EZNbVwCN3H8Sn/uFzeOymbSLJcAHnC1nmfTpxzUY1wHylhv0HDyFTKKK/t+TorhD/WYEukXQaWoH0vCxAsGb0AweGigpEdKZfAozcZJml1bwvMZlUe4cBgWP8+SXdaYNdrP3H2VjzI+Z1erBK/K92oB5rM9bC8rF+zJ84jqBu4JQyApVPtJupoZDPaprLanCzRhFTjWoc7CqEXeTTBcxUaMaWxiV/fj7CRAFb7ziEvtUpBPn9CAPTuxaCrtMTuOmOh/Hft02ikyogPbgCpTVnIBZJSGmDa4EIcocEmnaIUqKMT73zYmr4c1uIl0ywkyi2tTg7CIRykx4bR/BTlypbBW99pHYsgulWAye7RBQ7iMaZf5skqRBChzKfcuezgWu/kUm+9kg0R/y0yZkO8KO5k3ptugcr0j1YdtPfIXbeRhy76MMA7SzYL2XWGQUerR3B0+0ZpHoG8Bf//m9IFHvx9O0HNMequpbNcg0RGMVNoEcyKVcCetMI/HLWi0x/+Vl403jaNSnG5cTOadZEA2NTKAReuvFcRWIbAneKjhyyd2OJGtVzXGcJBzBLIXc28JaTMQRqBcXkfMfIzmvU5FWbC8ycFzhL7IcvpGLoSAeLTu+Zi1kpu9LqhkYBqeIhPayQChJlXPGOjXjqV5tR7GaQySbQt2wZYqkcVl25AdVYBntvPwwkO8itnEGQqinCN+pmvcF0+ZYfPo5PfflvsPmGbTqJiEzLoiNus7tSWIwncOjYBKZn57Fs2YgWNFVPSLThBhKRIpdRqqzhCfnzWFamckQePmyFcTCCxAn2N40vzp4xNyazHdmZuhYjf1dOeU6CVTI2ak2ZionNDTEUOxkl9z4aLHAcAa/X3ApaGD9zGXZvfwb9qbTKGvZ3tWkLBQ0MMIMiw4knLj8D8QKtd7WDOFAQQQsxNLvAa95/GbY/fxRzuwMMrouind4nK1jvrMjnVq038fYP/ztmo+uVJqfHxjG4Yo0OPa4JAlKScquW8fl3vQwvG+uIO9Fg6h62lIFxuJ7bivxslQPEyEnw4b/dnFsZ8g9cSBwYrkZDrHvbZYitHdQbzE9NY37vFMon5zF/YgadahOpTgTRkG5trCtNbiTmoHBrHDGNNOULJsWqCEnlokwITYRZR4YBlmUKeN2ztyGaKeLkBR+20SaiZ4yo0QDPYhr3LRxGJJnDO772TQysW4Hf/uQFq6NkMs0hAecWHo8rdSNowt6t6k+mZE7xgBtcZPZWG1XJmjBOVKXcwE1o1Lw2zn3JBs3JaqyRtbEYLWZHYsMFjHiWuhC8oOuA5lCDCGoV61OK8x2Eiqqsr0j14wnPoELAwtd7YpS5YMATRUqHyaRc5zTepRSqo0XE01ejctTI4uxmvSYXt3pzFle+/Xzse2gbcok0hlau4NGLtW96KSqdBHbfcRCNbhXFNQuIpG3OlvIpqhEjcdzw7fvwqX/6NB67cQcyqYxOWzKcpCXVaGB+gQGti207d2F85SrVf2mmyOKoW/+fG3ChPCc9KA1exE1czqfEGoUk6OQ44/LHZb3veMT+AGC5Jj4yyQgajjd5UgUtAotyBDRPJrUc9Xwc0EYJHefP5AXhWOZ5FZZmt4GRtf2YOXEAyRqrQ9P/5qnL0pmBk319BlnOVpMwoqEHBV1rMTYaETTjIV7zwU14/O79qE5EkBo+iVr4InKFJOI06kqYYTlBrGs+9FN0C8sQ61mJwqp1KPYPihE4s7CAVq2CwSzw1Q+8DJn2CbTCONLxAMTAqVbC9hL9mdJZYggkpjBL4MFH87Ikgp8Ux2Xr2YgAx8MOfrZ4FN/83idVGPuWrRCuIDBt5GaI+vQiSqV+qSgsTM2ifGIOE3uOIqg1ETZa6Fa6CMj6cYbYUozgmzrDQyqusiJhsPzAoaeQ7EQxcf77VLtIwJORKBrBi9EKbp99Aa1YAtd88WtY/6rz8MD/7jRjKKKCBDlEljAgnqcAbzYfsCIaTwApVBhVkX+fmplCxGlmsd5imsxTPpVPo8h2Q3YQSal4nNa49yWA09vSInIOBamkqWtI3lSiZcY+4ukraRtOHXWMQM7711PgUD/5uMaE8WN9POW46TUiF1JQ3ZwHJCpXr5tmcYNlwYLb+AHm52dl07nxNWMI52dRjOQxtGI5EMthze9txGwZOHj/CTTDGlLLphGmKCzAUTe7H1y4P/nuw/joVz+BR37wHLLprMTuuIj5fjK5rlYxOTktOfO+npIR+cW+Ms1iZg9ybjxlNKH767+I5PpTV9pU5CzTKlTgH21gqExBNUdrvSnrYEYSjeh05vvwuTVqRH1NsZGDHiLfcPrKPVcOlXgvKNl0KA03l0cFOtbL7TY2vmIcL255Gj3JgvkIxRMS4FP/v9NRz93PQiel1mElEnu99VYMYT7Apr98Be65YReCZgyxZXPYvvMxDA33Yu2atejr71cZdPzkDP74Qz9CmCshXhxFduUqlPoHUG1UsTA7j8FYG9/4wIVIR2fQiUYws9jGkRNtPPfCIew6SKFCUugIUBpDgt2JFf0xrFpWwoYzhxH8b2FlGOuEeDxawS/a0+jEUvj7D1yNs84Y1QcR/Y8JO2+6G5aWiTQb4lT/Y9Rr2Ywsv2RMz0b7QhURDq9X6xqs539bE1Uszs5hbnIarVoXlU4d1z21RQPhBza8G3EaLsWJ3AV6/ZOJDn4+sxfzAbDp7R/BVe+7Gvf8cDuChlERefrZ3GzDjMbI8W22NIvJjXSUw/Ipeseamj0jMvu4JBdwfnZuYUFXTV7uyjUrUSxkEDZ52kQEtFGrin1SBhyCNVJb0KQGbTVa9j3q/AaBshPV2JmMo4+aMZgZejnfYKZ/i/NLUbkupcmOGv5kJ8kLlptdDnu06UxaPRiYFUVNG54tphSqlZp0hDmFM1s7ij+59jIs7JpC34oxBPE81r75fBw7UcPhRybRDpoorJpBM2Kc5obkYUkLTeOOG7fiw1/5OH53024BbMWegtQReR1MVXnSHzh4CIOlQQwMDGj2laCeKW+a9BAXt3yg6EecMraVBTcT5OM94ee0oGHEDKua+Lma+gt7zWqjuNaM/68X92Pq6Gei6w3bmMr2XOeDypVEavi+Xk6HAUW1sPrJZhxebi3g1VdehD1PbhZYyFQ5kTCROZUmEjKI6bkxW/MsQQFFiRwGzhjA+is34K4bdiEVTWLDVSW02mZETtYdA8Tc3Dweefx5fOE/70c30YPk4Cr0rlqHbD6DykIVuWgb33jfBszMTeF719+NPQu9aq12wizaLEVpGs5eD0k/ThPbm7tFKHbAdPq7uWXhb4MKHuLoFf1fIgE2jPfh/33kLeJZsk9IXS8lJBQN4/51Y2Q8+ZQGM/+P2ryrTXU4epYgU1pTcrFTQZFN96a0rchSIkXs9X/xWcQjOew+511IEYlNxkV2JwVsPt7FLdN7MB22sOrS1+Gd//Jp3PPD5xFWYyIPqL4Vq6QriF8mXS7FJLrMyMnWglQWnFUj02VOBFFqhbS+voE+jA70C43W4IAAD6tXKA2zxBJzJ6k3h2ZU5wJhb5btDqZ+THH9VI8GviWMZ20I9ZmdGsPC/KLSSvYbGeGloOioLkojvRgd0XOaPXMYvV4XGGfpvpFeOBNbq1ZQayziirechcb+eYyuWCVdzHV/eD4OHC3jhfuOotibRXr5CTSCOSG4YbuCarmG3r5+/OJHz+GDX/4YnvrJbqSTGfV8+/t7tQhZA56cncKhFw6jVOzVxpV3UoIgVsbKAVd+SPliadzRgpa8kJxgAfWrubl438yDmcGTQw8mSqBa2pVs2szOo9dcDttLhtu+zcTPLyqg0mMius490p2cDBjKxpzDngJMB1iszGGhMY+RoRCxWhcl9q2jduJ6mx1mEjIoo6+U27wMVJVGC2tfsQ6j563GPT/ei77eHoxdyL40Mw5qaidVcbc7EXz2S9/Bnb+bRJAZQmpsLfpXr5a4QHl6Du96wzjuuv1BHCxn0Y2aQAFT4EjUAoyoyQogRiVW1yEeQ8vZzqj99vO3vCn89+eewo7j80rReBrl48D/fu1TeohEUHliGY2R1WsEMTaDCc5EEppEKRX7kMwWjAXDiEqLCykXmJWJ0haCD+VF1Si84fVmFfFOB+e94VrEC33Y8ooPYHCyKlS7oxqpjXoigt/MvIiDYRmRvlH8zU3fxaN37kdnhhs3q7qT18wNzEXGB+4XjG/60+OGpywXDq+BYmDsPVebNSxbtgzFTEapsbxz2GoQsOK4yi6VVapKPqAUEu305P2gYiSV+WUKzjS909aG5EnFfpxqJKVwfsvMAAAgAElEQVTKrI8M9eSC6usr6d+46dRycEPTTN0ZeIiHCGGNxnTikTcrEQMnN0N63uz0jPF/K2VUqwvoWxdivNCLlWPr0GjGsOHai7H3wBwOPjqJUl8BtdwOpPIEQIDjR19AMplFqbcPv7hxBz78T5/Alpt3S962r6+oUUWO2c3Oz2F6fgZ9mX7kZE+yqDqcGQ1TN1E8eZKRZeXacX4+l6k4B+D5JZKFPIGdSbmb9eZn5Hog44nsNAZ31k/MMigqV6FwvVJjk9S1DWwAoszSvIWN3OxscwuHSNsJr00t72DLykh4oAZ1uTaH3qE4Tp7YjfHSiNJ/b5rOZ8uSRbJBZLWlqVNNSZsUFisVXPS2lyNa6MFjtx9E32ABwxvYozdRP1qqRoOkyspL3/ghLGIUieIo0ivWo3/VcnSbLRw7dAzh3CS6kSwiKQZz1sSWLfjxQ3M7sC9t0qXx19O+9+SN/xA+u/sgvvQfN1qNyRQ4AvzL59+PsZF+pAsFFOJ59GRzZq4cJOTnU919GIdvfRCpiRpirQCtiOkwsb4sNQIxbyS33WijFQvQoWp9xB6wTheO/kWjWP21jyJ5yfk4/NX/Ree/7kSE/jsBeZ6U34/hifljeCKYwUK1jU/98LtYrBWw73FaH9KuMo4ux8SoPEH5DzfMwM3Hv1MqlL0dyqUeP35cWkp8XYqDnH/ReZg/OYtChu0Mi+pSqHT1r2aTVSdZFjE3M6eNwpPGo5r8fjLJ09xmWEn898ytdov9R6NecjOSyUWQSX1OCagTOeSMqtV2xTz9hLpakETfuUm0gBIJnezeHlM9c0m+kjwxoxp0anYSzdgMXnXRWiwfWodqLcC5116MFw7NYebZBhKpCCZaD6MRziLoUG2pKetIBtX7f3kIH/rKJ7D5+q1IJTMYGh5AEJBAwpS4hrnZOfQVS0of5QoQYzCxe5FOmqQvN2ahmNMCkwome+y8p3QUiMdxgvO32gQcmrd/Y4uJwZZf1WrD8AgOs0fNq1g9cGk2n6I18Lmq3ylmElvipmjilTL9/LU5Kphel1h97FKwd85yo96U6+B8eRapUh25bheD2Z6l8sXPpMtrKZV0puP2XNkfvuKDV2L7jhkc3VHFslVFFFfPL302ri/yJCqtNl53zXUI08uRLC1HenwdSsOD6MxXsHPLVh0SsVQKMRcUlBI7PTYBul7uibO87A67coT1uqE51FW+6R/Dcq2Nj3/x69i06Qq87hWvxJrly5GqVTBz12/R2XscwZEpxJpdpCi3QhSWi0+9XIs0GrbvGOLpawJC2CJekwni9GHZ/mAkdjsXrW4bfVdegIF/+yxm7n8alQ98E22ieNTNZV4Ti+JAYx6/qh9CtQO89Qt/g/WbXosHfkiyAN+fpxJnNbnIynr4WuBy3DOJU/XhOmactFgpi0zx2t+7HJP7J5Gk8zd5xHSrkw2Iobka5eNwPRFOESVSSCVSJiymuo0zoQlDJWWBZLeTI4/8HUb/VDxp876UanGtEm8JyZ+VxpLukVH95mZmxDUmsslTtJAvGFgjw+cKkjJutv6lpYddCdNxU8zMTmO+OoU3v/4s9OeXoRWmsOGtl2D7zuNoHiZzDJio349uZEFpNgXIZ6Ym0Vfsx7anQ3zkKx/DIz96HoVsAcViFvk8gbEK9u55EaPLxjTN4wVEeL3SOdYEmPlIibXGvr3bbAqCTO2oXhE3v+AKaZMLiwqyslrRYL4NgdBPyRuGcXKKtaz6x+Q+M/X1/V63WW3w3U5gm5F2rbTTZIWZcUpUPWrcaG56Pj9+n6c7sYaZxTm0g2M4a3Q5MtGERu24ljzST2tSormsm0mznCrP4M2f+n384odb0F8cw9gZeXSyRzA5OYnJySnN15JnX2kA//i9R4H0CFL9K5EfPwO53iKObtuBxfl5pDJZxPjaMbo7OuNylRqm3qHzVlguZQad5KvLArXOeAo/f/t/hfmFNo7evwOTjzyDnmpHOsasW+Pqldqu91/EakwEnQLddnr6qQU+XG1cZy/CyMeWiixCNNnvcngLGvLabfVlcdbm76M9V8exqz5F2yGdtCzW20GI2XYdty7sxWzYwblvvApv+ZtP4/4f7bGBfuk/2QynGTTb4uHDZGvIs3EYwVmbd+MhNr35Amx9bCtKyX6zX6Qwmh6ODczzpDaFhLZR5UQggNo+PDG4qZge2khigGTKPVi1vgL1K0ny4O9wMUpkrWvADVM+LjKBTmxZKTW3jVivlDWr2kO+cSajFoiGxqVKccrSlEHSt4p4ijOVnjx5Agu1Gfz+G85BX2EE7SCNDW+5BFuePojudBKpeAwTzQfR7syZ92+jiXa9hhNHT2B+cgU+9o8fxb0/eAY9uQIy2Tj6+3oxMzuFWpmqjD3i+VqWxNPALCK1gLgpnCkVsw1D7g3x5896XjI/L0sE/js3r8Tb2PtlnSy/J1L6rBzj4mdgYGqr9hDnp52ihaW/RkYwn1pj6p1Od9XoJkkuRK3dz3gxRBJYTIaojmarjonpaVTbR9Gfi2Mk14NcIS91EqWstGXp7dW1skzgfHRQiuHyt70Kt3zndxgeGcNseyd+fuf1uPbaa5BMGn2SG/fhJ3bhB3fsR5AdRrJvBXI8cfuK2PrAQ0hn8qIFxxm4nfSP8AExv8wzyXVWrWRz3AdN5y0N1AQIHlp1WZgkYOEGdXkTk2SdRLqId4EW2xrgrKZXdDTNV40guRpQObgWIAegqV/rHP9MCnhJZ0onhtNf9qNK0WQC4w//B7rFAg5d/GEEtRYiBKjULgpQ6TRx59w+7A9rSA8N47M3/w8e+vkBdMuExTrIpvPaELIldBuDCLMhyTz1SGvsoN6u4aLXbMTBgweR7GTRqlcx0DfgVAbsQXHD+tqYf+fD4BfbD+w/q+6MUxzNUE2zrjSyvEYB6ffSqIs5RcoaU0WemN5xQMCDQ1RFPCM6TUmcRgP5bGZpookbeHzlSszNz6NDcoK4z+bB68GgmdkZG/RutzEzexLHThzDa16xEr25AQSJPM7+o4vw9O8OojObRC4dwzR+R9MPMdPKtQoa1TIWZhZw9IUiPvqlj+K+7z+JTCqHwaEeCabv3LsDq8fWIJUxQQKhuKSvpsxFnkGRQUci4uTyOkM4s/uwnrfpGlvQl8xrta6NwI0oUy4OprSYXvJpm9IF00ZmQCwzCGRqXWqEzwKcHywxhpJRHHkP/DXye2rPxR05hKi8K884LskMi1KxxEOIjs9WJ1DvnsBLhlcoaKaiCdXjXNK5QlG6VBymCNoRrL3yLORXDOPuG59D/8AIUkMHUGnPqvPAykrOjc06/vP6B/HYvgCR/DIkB1eiZ+U4svE4tj3xGHLFfs1gRwisatzTmQIwXXakFTk9SkbJdL90ODrZGpvkiyB4bOSCkLmzmQrZEc1tlzDW4lIU5QtJ7cJtUJv4M5sRRUSZe7kBYPVs7YubnI10bmhX3ToFgq7QaS7ske99FomLN+C5V38C2dmKgCARyAhUBQEemj+A59pzIof87a034unHJtE8mUWM9Q0nPNwQv1BhN963JGcTUrWxgqF1vQou8WYcsUQMhVxRtZTUPdyDZxTnBuHn5GmXSZPGZ20HnsBcOPwfr5kbyMQHyCWmf2qIYq6gHrMWdYcSLaS3LeqGciaYwUS9RYeAsg/LB2MuCHZ3fCosAbFuF7lMdqm9UXdzmyZqXlcdTDS2Vq9gfn4ar9y0GrlkEalsEev/6ELcf9cOYD6K5csHMRt5TlRJ8bbpbM/yodXBw/dO4+Of+wgevWkr0tmsfIlypTw2P/woXnLWOTZQTkIGTzFxj01xUKqMGiC36yZQaIi6Dbir1SNPZDt5xc12JwzLCdbTzBjUI03EBdBQmpWL0p/U8qJyLR1OMhmvm5vEXlM4iAsMzIJ4TRL386m8a2fa9BjUGzUKp1F8mTpPLUwjPdBBs3wCq3IjKknYseDPkPvNjIKOgCQcXfiXl+PI4TpeeGoSgyPDSI3slN4VT3c+V5VkzTr+4Tu/xY5JttPHkBhZjaHxlTiwbZumzRKZvKi2HDf0paWBbJY58rqYbfK+MEX3AVL9ZMe00+bVxnUnqMwTnAh1zGECPpIpHQmApEvd/MZUX46ImtIka6X4o15725v8OtaPT1/VdHepTPHj16D3L6/Gts9/F4W7n0eXyvOsYUTyCrG9MY2HascxG9bw0W99DdnhM7HjgSmZaVGs267B6hx+eN+096lvmKhj1dljqJ0gV5XSownzi2kwdbWRRQYWTaqIZ20ax5qPlCg4QRHbSOpZaqInKU4t68eeYo/olLJecWimVQx2Shjrpu5SLlNL5KkwMNinf7f3si//Hj7VXJxbRG9vr4CoQr6oIGR1HeVW6vqsrKXn5iawfl0By0dWIJZM49xrL8evbtmCYtCL/sEcFuO7KBJqI4bMJIjyV6t4+qkG/vBPr8azv96rdlCuJ4XesSzKxznwbm00qmbw3iiu63rtWZMRZpkJkXOr9atUzHQlk2rVGlH0viUQTlM6uieGMHswi5mMSpKWnaDKdCRiYJuXmAC/L0UMJ2jnUWX9V2xdu9c61V0KTZEEn0pzuoeKJJo4Yg8dXTHDphYn0QgP4yVDa5FLc+M6JJktwgQ7FnU0unW86TN/godu24OgkcHAaAnl+GOg7JJlXJZddFpVvO+6X6OaGEaydwXSy9aif2wUzz26Gf39A4ilMzppSSM1BQ4DvtgO4p89ocjfJ9IiPdXWmGGGnAdPLXu5Nq5OR9cz0kZw43Kn6lc7Rf3MrmDqUwerEFWfFnkyOVNE9TCdnIyG6ZneiN1k9R7TreKmjcj/5ycROVHBsT/4AkJasLuJGb7FyXYVt1b2Y7pbwUVv/j38+Ze+hF9/5xmErUByI0yrPEe1WOxR6snWij5kpIWL3nQODj5xDFE6kDurTJlTq/fLn+NpYO0ev1i5wRURXUnAFJjvIzUIjgemMzqdqVRhgZ8zk9YaUW2mE9k+nxHajVRB8gY3Ir9IuvCBj3PK3gyNi8UrU87NzGsUkWljJpMTpdOfSLZgu1goL2B6agIjQ1Gcf94GsZxecu2luPWm32Esvxz5YgTl+A50A+uVtrvUvapJA2pudhg9A8OYeHoGgwMDiOW7mJo9ieH8iGpQa8cwZbU2CVNWzchKLN1ojRokQFSsLvV/GVzabXMSiNiEFH+ezCWjjSY1tOExDwZHsqT4M5TvUYeAmAB72q5V5x3rBcy5AOrTaB0QmtKyUkQIshsEIW1QCDixBtrKMP0mv5oYAi06W00szM1gsvEiBrIJrBkYk2WNTjzO7VIzLR7H0IYhnP36C/Gr729Fqbcf/aM0VntCdS1benJdTGYwNXkC7/z8LxHmRhHvW47U8DgGR0ew9+ktKJJVxdOWjgsJTiNZhsD70GyTi2ClGfeSZwNKtsdbazqXS2WBW0Zfru3nj2058vEGOt1jc9WzNFoTREsypwR1bMSItYw0hAnXMy93spsEUsRNdv0ouRfoxvP/XQ+Q85lDJYze9w2kEgXsuewjoNUwwS+pOyBEA13cuLALk62qdJW/evdtuOfGPYg1yAv2UyVRpV48OUVamFtEtVvDm655FZ7Z/DyyyQwSbLS7E5k3SQU/f96JbJvyhbsXztBMCh1CJCmYVkY2m1MN6GsPDVArG7EbzM0t7eC2qX7wgVYWFxS1uWFtEZtIGiO737iq37xxmrtGKlTy/fj6DAILi1Wl3BxlPAWQUctpUdTHZHoeF23YgG4kjvPfuQn3/HwHBhJ9SOYC1DI7EEQoisfAydqwpfo5VTgXEweraB/rCkAZ3zCKY7snZNZlz6qjU4drgggwA5ykZyjy5nji0jB2QxzS+2Lv2g0fcMSEr8O61Zip1ttmj8bqO9akBgoKdCJgSe4320cJ07TW4LjqbFNT4cv4UT/7Hadppjcw6SANqstnmA4JnB5qOjM3Xrcx1BjcqTDZqDYwsXAUtfpRnLtmDfIpuiPwVEyimMuJQHTRuzYhjKVx1w1bsWzlOIL8EYTJSUQidr3iTXfaqHUDvOPTP0OQG0V0YBWKo+OIxUPMHJlAtm9AnRKbCIuKjimchLRWlWI2fMLRWj9wov3oWGgCsPT5Q9u4OgUdxO6lXsTY0H0I0abDPJFibl9fx0qmxrjBegAauHYCc6KuWWSkNaSLDEsnNL+/1CDniVssYPj2L6PS3499V30GqUqVk6+ajOjwwXY7uG1+L17sVNCMRPD3v7wJB7eHWDjYRk0Cb4YOU+jLZESZZDfwmj96FZ5/8lnkUgVNuzC4MLDwRlMwTSi0Nok9SC4e2o1ysRoZg4CKtSxIOuDgtcUt6znqlHdTLp7mp15mtQYuWHF9azWUeou6LvNqtTaG94IxQTbz1zVAoiPbDn5fPWNJqhiyXK/ZCKM15SOYm5s1KZhqBXPzM0gXFnHROeeh1uri5X/1Wtxx/e+wvGc50sUoKqltQMC+qaWq/Awc6B5ddwmeu/8wEtU8xjcOi0dbjPcYi8xbmDoqIe8zUXXSGvllFi0R3SNeL+WKfHvLVD5Dsxh13GbrRds9NwsWnqyUJDWgy6fdIrQwhXTaX+rLcrTSrRsCWkJYnTqkP5F4Xww45FqgTWdCyhFiWAmLYW+ZiLQJA+rnKB7XbGChXMbxyd1Yt6KEUjov76BcOidKJLOnTR+8Ant3nMSR58soUGu57wDaUng0NVQBYN0Odh+exRf+7QEE+VVIja5DaflqzE8fRqvaRLK3T9x5dll4/WQJ+iBH4pP65Kdlrr7T4Q9WtsqUHfP/nhq6QN5BYn84Lx+lYFKlt5tHaqLsIW0f6xdtusMI/qK2ufpORTSTNd93cv64Ek/jQ1JUMSKXAAYytXqyCN5xBXIf/DPsfc9XUdx2GKGrMcmkYozZPHsAT3RnpSzwse/+C7qFVdj36DxadfJjCSjZbCW/WLtcfNV52LF1J0ppRx7QWCEDvfWa2QKyFMsQZY+amqAYh7TrOiWLhaJtNvn/2KnK00AGWg0j2osUQMnXuBFBuCEqi1W1pPjgyfbhIjVE0NXMsjqpqHfL7wlkIpHekTG42LgZ/ICBwJ66aSHz9/h9gl8kQ1TrLczNTyGZncJF55yPVL6Is992Ee67/jkMl4aRzHTRzO9Bs0WXObsGRvf52VksO3MTnr3jKMbPXIG+oTwWDswikcqphSTwx1ExfW+T/GTW1MwseLKxx8375a1rFNYc51jZBck61YrWjW1cG7D3X6o36zZIUOrrXQpexAHIIdYGVWpLsoXJmfrSTkir62Dw2fN+SczeqbcYW40kDL+5DCBV8NagekcbmVRcDrdPTB7DzPx2XHDG2eZkkM4hmc0iSAa4/L2vxYO3bUdnIY7ScB/i/XvQCo07zo3rg/h/3nAXHtnZRrJnLaJDKzGy9gzs2vI4Sn0DiBd7FdxYz6ssEOEkpj5zwDlhmejBJta4R5bISjbUwnvpeRLBs6MXS3PK+wL5h8WXMHBF4PFSrcdvmK6ytoHzZ/HppRG0pUFMdUd56FqqpBNWEx2urcSGrUuXooko4meMYeDGr+DQz+9D4ut3oJUIbIiBvOVOB3vrM7i9ekA3+8Lfex2u/tsv4tH/3S+QhuR/EgsicdMzHjt7EEi2ML+/hnQuiUTEGFGGk9tMsdExzUTZQ+/sH9oYmRHjGQykc+TYTdrwrs3AB6bo6NJkntr8nAQ7uJDJhBK7hxGeSn6uByn5W6dgz3tNEoI3txapg7alAmH48MwHlq9LCmCrzkDH8bgWFhgcSPbnMECljoXyLMLISVx27gYUV4xi3ZvPxYPXb0OpNIBkpoV6ajc6odHzOBjBz0qlzNVnvxI//taD+PQ/vxeP/fQpFLI9qv3ls+PS/6UA59M0qydO8YOd+L0tNmOK8TPa6Wajn7z3XKD2/Lk2DMziZzMlDVsjptNt5RWvT1iHq/kM1OrqdbSAtTh58jeEa7B0s3LNnrMnZ3AjLAGObhSQPyHMgddIZYw2Qb46dh17DGsGSljZN4I412U8jdKaEi6+9hX45fe3Ih6hYF0PUNqNbruu4Rpz0ON67uJjf38zjpSTiBVWITG6BqvOWItdW55BaXgUAZlj5D+TlEIEmZvVMdKoeWYgccRQf5YFEac9zcNL/043DGJGAYKtIy8/JRbnTkneoBhrU4cE+5NCD1CkDIuYlmqae7g2tJN1JaTO2VprfViPkzef56wHVlg42AO1Af1EXwH9d/8rYtUu9r/hsyJ3sNdFyUve3JNhHbfM7kaVs4p9efzDnXfgwR/uQyZOXWVyUFvSpx1Y04uB0T6UJ+jDQqmUMvpKTP0c2OSmLeQzG7MmPReMQCWJiiVMnFojfM7KwguZuRPaVB1MTpWDF9x81BAyj1x7KP4UlxCBQ1k96YLXKxYPJYGc5QZrMVIifbrnF52eBetxPtBGS71QlgIsU7jJJyYmQLdDMoGmZvfglReci8L4CFZdcQ6e/PmLSNIwLdtGK/8iELAt09CDF4BDe8vsejzyqx141yf+EIc2T6gVR0BJ7BwnfSt0XsMbVOPIngZOmVay6XrZXK5lJ1zEhj1QRJ1fKgeEbVjqyr1FUIe/w03ja2Kesja/a6kjnw0BJVtHlk57tVCmzEKl5QYRA0XTddqTwdRsCzzk/WdQNVzFVFGMJmm5BK9loWxgGjf/8YXDSKcmsKa4BslsHKl4GmsvW491l2/EL777FDLZHEbGc6im9iDomqyqyeoyECziff/vFiyiB/He1YgNr5SiSKNcQaanF4l8QTRfL+fLtNnPWBN38Iw9May5lxzeYofOqUCnTb997NLQI1hEkj2rxxMqfCrp20I+yWFEYP/Nn2AOebBI1zUtYf2buzn8M8EQf9RbAmyRkUyeZUNDKP73p9A5ay12XPIh9FIbi0U8a0m2Gbot3HJyO04kO2iGdVx35x3Y8tAMwlmDzaS4H1vExks3YOaFGW0ioqZ8h9mZOZHmrTfm1SttzMu3I5jSSjZGd8gWmAm5mXyNMgbWbY5AwpuptFgqDVTEJ7BlWQi/eLIYD5kLlUHBojK9l7hYRNhfLKNUooyrnTys93p6Tuk6GzvLakL+TmWBKbLZiPhajekjpT752oeOPIerLtuIgTNXYPDiM/H4z3Yimy0gmW6gUzygul896oap53O079jJDI7snsc7Png1jj1xEulE2gUfA4P4VXWeQAwUlm055wtHDmDQ4joxYNBOTKs7Wb9aNqa6XrO1liG1HEXW+MWnnChIwOCz86eu3/Q8xetSyLDX8/8u7W6Bgk0paSylx9y8TlGS18UAGYtSY8oZRPOaXI3M+tK7O87MzePw7G9x9tBq9PYwkMbwpvf+HubbIZ781SH0DBWR7VtELXEMQViXtKwtGTLaGnj3Z3+GTqIfmcEzkBpbjemTxyTQx42bLPTYmJ6mfeLamL43K4MMch1cGaOSSlrShgdImCAwfWUNmm4feXl4qgi2qGSwtJvGcI1fqyu4QSxD0Wnj+r4Wu2yEzVpJdkrwxrHuM3DAjntLdwzU8GNUZGkN5IqIXv1ypD77V3juqk9gYLYhoriiI1sp3TYemD+AbcECupEQH/vRf6CDFTi0mT24kKIPeOklG/Di9gNIMd0KIwpCSkXCrto+kuVUe6PtLCdYn51Sm2AarDE0pb8eLLJUyNfmekpMs2ocjK8jX+BgudrmOn0NYQzQdhGfC4r3lAuaG5lUQ6tPTdJUJ4joeSbnygejf6OKQpVStTZULgvGtg3b8/e5IaSEz5Oi3cRiuY6F1hQuPWcIoy9Zhb7z1+PBm55BqYeDIh20Mnul9MCNR++g2mIFYTSFp5+aR7cM/NVn340dv9wlIkgu16P+NEE5kd4J7DEIOuKCyY8aCczKB/PbVe1GkobQ0oQGJnhSW2sLyOcKCmJ+Tla0x2x2qe+qk9hZ3XCteBMyOw1t8ovvytdMJ1Ogq55mmsnQ4sL3eINM2hg0TJOYJ7G3pzz9JNe6dVkin5ECcbWGQyc4mzyPlcOj4pxf/fE/wjNPHcXUoSb6B/oRG3oRYZScddbTxuASyFWp4z1fvBVBuojU0FmIJtNoR0IkMr3I9BQRTWfVnvHlmW1BZnYxE6B3Na31cO3z0J/JU3gpV2RYTATB7uWX+oPP0juS8qWImHNop+kpaac7cEWuB/Jk9U71tnT5u+rziQHiCnZaUbqJGp+WKgR4UEi1TQulbB4Lg1mM3fFvOPqVH6N962bz/KHyA8fx2i1sb81gc3NC0z1v/9cvYtXZr8JTP9uNdG8O6zesxuG9R3RTmIYnY0nN2JpfkW0QpkJyqKcJssbkLKAs8V4dWd1HdC4kXic3I3/HpFMa0olmmqcb7ni7ipCyhHSDCm5I3BQdrNerqB9ACLWsP93pLlTcUdx4GlEgTf1TaguTsU7pVf5OpS7wRWkfn4mUIpjutTA5PY9KdwEbz85j/CVrUdpwBn57yzbRGAv9ATrZF0z+1WlwVRfLCCNpPPrQBAYjWfzF378HT962HYl2QmqDYtPBTMD0rH0dq7TwNGacJqtaUr3wih0e+VTG0ek4i1XTRPZZhA+ACvSOJWSKkdbz5QnDTMfzc8mqUkakn3X2ma6OVr+eo6ZsIaq9ZKi9rlsaxca29wFTAcBlVabfXHNGajT/aqNaKWP/0d/h7BXLtH7e+sV34J5btiMV6UWxlEe3j8bW1F2O65mS+cZW4ez0At77d79AkMoimh1BrVHD0Mq1CHL9SHL6i1hL0vAWyxhs4yqbFe/aqJ3iO2jzdtGVbI2RMyRpIWvbLoLdY5cuORn4Rrnl7ZYGKyWkgqH3u3WbTm+oOsZACD4AzTA6cXR/QT5NUprqWiEmoO5qHd5URaEIYqU8Vt77bcw8sBUL190g7VsnbSTPmqPtMn5T2Y9y0MAbP/8hXHTlH+PuG7biyqs2Yd+Oo4iFEGXN4Hb2vCgVyjYCwR5OACUNBVwTb3QAACAASURBVBZTxdIbayNxkTjK2WnUQxMbM7IIPyNBEYmOU2vKjZx5fWhFezkeGEBC4gnvp05HTcLUMDg46OZ5rffosQJmAn7OV/e7YsLs2iDRmJ2ynHBp2YCBmDSRuGprkvZJAaSlRbnTwDkX5TA2MorSmWvwwM1bMTI0hHiuhjB3wG1cowmWFxYQRpJ46MHjOCM1inM2rcUZl16EF+7ag3KVxmj0ETIFCGPu0GjMaXA5Wqef3OF9phm2v07dM4chMHiaLA3rSjs9fGlgizO0ckjgyylfKqt5rT/MZ8ef4wZRf5ZC7sQiWM5wnJJ9Y4KhyugMe/FglzGv7NDxPV8/oWROF6HOH95v/l0Cdd0AR6cOIhudwdr1q3HFe9+Au36yE+lEHoWBJBKDvJfMTo3h5dtRB4+dxMe/fCei6TTiCTouVDEyfi6ifSMIqJsdT0i3mffJNqsRaLS33OGydDg60wD1fV1m1glNxlbFyu6xy2Wz6dnvYgG5WGARsKPepi0kk8Rc2pRehoQbXBMc5tInbWZPtnDRWUgjZTzZ4nBK9fwzazOeIkTQSvkChh7/Dqo7j2L2A9+0XJ7TKIyW7Q5muw3cVjuAxW4LL33HlXjt296HwexyPP6bXcgQhEmZUJdno4gho+a81Q6iw7m6kbWrXvi0TIJPXOkfb5T7XZIguEDYtuFDVt+NKQvTadce0qLUInR1BFt6ra5TyDCghikh081Oq24kFeatdFuv17UI1cAX5c9SS2YHZIEpqGh6hsCSSZuK/OECDBdQo9bA/OIC5soLuOLtG5GLhYiWhvDQT7diZNkoIqmT6KYOgw9eny/oyn40CJJ45rlpjAcrkUkmcOk1mxBms3jx1xOoo4pItItEGENIdQZZUHYQ7TozNUdL1MZjuuwGMvQZ2i2d1Nqg/kQ5je2kZ+ACuQKRo/rZgeG7ECxvjEHlBc2ZLtsYnAn4i4rqxAmWxvHcbDXXH19bBA43G670O8ZAaJJA3PAyg2sYgYanJw8RBt7JqWk8u+VuXPO+N+NlV7wcD/3sRbHC+saSqESft1ljR6Tgg2SgOnhsGp/8+p2IxTOI0Y4iFkHvygsR7+1Hh7PeZJLRtJxZmKWd+nzClVygs31oJ7F2JX/PeVOxzcl1J/R+z/JNp/IehxT7COVTItZporsJ6fPo8almsaKc4wsL0nZv6us3f4PVMA/ow5IU/Ywb2G5uG41uB8v7B1H4zT+hOVPD8WuvWxq3s/QOmGvV8IvafsxHWlh79cV4+0f/HlsfPILeZC+iEfbHDAkXgun6tdLn9Wn5Eo/YWhbyQfVyK6fxcDWvyeEAmkUXC0Zsd+LmYgZpUsoCgp/g8Owp3h+ioNXFiphRsiBh+8MRDKhW71Nj3ikuLO5BSqVaimj1Ne+3MaYog2qRWSqJAjSkD+vaSkTTG3rwi9VFnPfmcWRyUcxMtbHv8RMoDZQQpI6jGewz+F5JGXv0BDwCHDpYRW9lVMBNN9HBS990HgrLVmD3nftQmaUaYwJBzJU/zLAoYObKAx+whNTyfy7NzWSy+oy8h3SC8Pffja1YUD+dyHPa9JEvT5ip0AicbTCF09N+3nAS27Qee+Az47NgENSn5HpUIHTDIW6V83eNd22ZlhFvDPlWQHTWNvze0SOHMHxOGhe87gI8eOMOFHvyyA9XUYnss9aNzMpPHWS79h3DF75zP0BdKOIRuRzSw+chmu9FLEcNK27cuJzo6VniuQMKVk7myPxxA6XiKpe6xlPQHtAZbZs02Ltik1JlS1+WNrr+7ml9HjRQu8RB9aYaYVQvnzb7B8oTwvpN1nc6PV3236N8DE9Gr1xB1Hi4p4TBn34JtVQKU396HQLnym01UxQLrTpuLb+AmWQHF7/3arzkgj9A7UhWxHBq/LKSsVSsi2w2s+Rw5pFkf6O4WQmc8Ob4z6h0x/VVGY2LPTxhnU6wd2Vwo2QUaGMqafPHlkZazQTnWdRFf4lD8fYeZOH4E4DyJYywBvQYuYDXayoQnSWKHj+Hpm3o+sBUVSvXUmV+JZKkQrpB8m6AVDaDcrWMNVeNIozWcHxXGQefPYGh0UGEycPoRg6Ic8yNG+XIZtxE7SrTDVSOlBCPZZCkbUw2i9zqJM561UaUJ5vYvfkFBLWkVBl4DU2q7bsMw0zHHNWz01TdLz8mV9fq+p1mlB9/VOotewNPBNE2toXp5I7swCBK7Vp47nek6OgIPD4dt/64pY+MSQQM1cryPyuk36RX/X23zLGzJAdE8I3BVm1Luhh4NhuDcHYCG1+zEfddvwOFQgaF5VMod4/rkjWwIA65qaLs2HUU1/33g269A6WBMcQH1iOe70OHBtmprH6Hp2087daAH+tzhgOWevvDkWm8gZW6fxF/KAUIdoxcIuaUb9N4YMZQ5FPyofqg3KRuQkhC4K5G8RtXN9ydCL6INgc964fyQ/ovgjq8UaoJw1Ath95SCX3f/gSCdatw6PWfQqJtg/F6qEGA2UYZdy7sx/FUA+/73jcwfzyHZKtHahFcxAQZ1Bvk7zj4W5HX1ee8Po/kMoAwHVUEdEZT3pKT12u1sVHiuDgZufV9iZbbtBDracmKhAQ+TDyOBHUDUMzvxdIxN2rlepCkDfL7cQq7OxE73gu2pHif/KSJ+qcUQFetHrd5VV13c0kAT2qN7GV3A9TbC3jZn23Ai3v2oXqiiYkd82KlxQv7EUanjLhAxDcWaEiC6d7ciSlM76Xsar/xp1NZoy4mA/Ss6sP4xmUaQ6vXotj71CFUjs8h3o4DHZ6yvCd8RubiTqoFRQAJDPr6mOORzA70HGCnndYDw6ysVt2mk8gawSwG3axlE8qcLEngNYl+q6EGYytJh15kC1fDKkMhU6umZ677tZRJOdE5x5MXJuH48nwdM9kOsFit6NSWiigNrocyGDozhvv/bxcGh5ch0ks3yZrxn0m66YZuVrqNJ57Zj2/c9Fs0W1QETSJJadaBM5EoDSOeTCGayiKgeXgyBRYtTIE9wYbrm2uB18z+tIIz1w4F4pzwvxqSrssS7FnOGveUIJXfuKf/ly/CByFUWObXRqZYSkmcRrD6jS414c3kw6JQuPp6px/nLsbyPZQSqY61xTn89Q8iuPRlOPSGTyPXcmOCtO9otzCPJu6c34/Fnjiuu/NWbL5jL9JBj5QCeSOVUrgeIk2lWYP495WcqNNdVr2rVMren5uQ+lS+Ac5/07ifs+10B4K1Kpwxt5HuKXQW00A235ug1RKoFNhp7TeiT8WkHsJ6qlrR0IOXOl0qRVyNaKdGIIEzWb6I9GLfU3bkUkeiokRUCfxU81Vc/ofnY+fWgyjPVjC9awGZQgrJ3n0IIxxMMPUInrj5Ql4LfG5qAhM7ExjsWa9NyAkXm0VmfzSObjxALBVBcVUay8Z7kRjoRTpGzKOL6gJQmamgXWmhVWmjQqvQch1RyuxSmYQ92UxS/GaVMV0GNNNCZl0rE2s6CHAZkxK5pPllLTC/vvg81CEQJ4A1vu+XG+XWgoIBTHxG9P7VkL7zHGJ/l7PAqqdVG1Nvm1NLTlCO+obuvdXB4KQPSxwy/XozOOOSHvzmxi1YPj6Cbv556VJbu8okYw0TCbHrxZO47tu/QbPTFc85nutBduBshNmSAKsY0WZiAWSmxVNyP/AYAWEufg5+ziWlGAES1t9VOeJKFB1Ep29cf8r6k3aJLOFOTZNYNZ4rbxiNlJiqqLZxTCtLfE7l3F7027+mpQJ2CsoYiZQzUgMYvQCs+fjbkH7/n+C3V30UK8qGVMvXp93GRFjFXdVDaPQk8LXN92Pzz3ehlB50DB1rm0jIu1wG9YJ8veOjrrSgXL1gLQMzxubm42fSxpbVg33JOtJ5lRrybKm/r1dVL8m825zn/eSKofM8BZymFJlEro9NYopNv3A4gGbOXMhOtYH9YpeeG2pJdNrECHTiO/oogyhPNqZ3XOy9Pb1YqJWx8ZpzsfPp7Yi0E5hemMf0zjn09GcR79kDRMwzSUG03VJmwqBVWZzG/JE2wuoKFHIEw0iJTKAVcMwDSvOppdWlFZVLtSutefSvGEJxKIV8Xx7pfBbRHO9fwnSOSRqIJBSYEMRRW2hgenIetekayuWGetxBlfeS12IBlKNs3FynCRwqoPN/3IBMmy2F5J38/7P6bE0ZCGUDDKauweOWfV6eYr525ikrySKHJ9izshaNmXzYc+e9oa1KkIxi7aYSbvv+Zqw9p4ROcr+456daVoZL8HV27T+Ov/v2r9FodVHK9yCWzCPRuxpBth8R6pOls4hQNlifk9pqrsxkXe2YZsoKXWnFZ0X7Hz+UQIM67jdNtu1adlloub8tSH9TGA2NIma9MN0uQdTWC1SN4WoypsAk59uiMzqg0jn1Ak+dEl4ZQYigkzXh7zTCNuokm7ebGLzwbIze+GXsuu56pO/5HbKIo4Y2Yh3gueYUfls/jp1hFTc8cj8mJ7uoH+CiJwOqjXzBxL2Y8vLh+S99BqeeR+6sCOzJhNQdlEW0O0IUJZXqanuri63u0kkrzV87qWXYRITcyXiyhcAHL860U4VU0POMKC48ybSaayBTdD4UTkWRgC+dJFfHGVhCAIs6TbWlsUiJqUmPyaReI0EcKVJOM3GErS6CVUmc+fIVeOLmbSiN92KhXsb+LQcxPDIK5J7EYnlOWsFMfPK5rDYJwaN6dR7tSgUTe+LoyQ0hESfRnzO7fPYkgiRtskbsMT5jprRc9xyuoMMhrVhsjI/3Rsg50WvNvtaRHo6iry+P4dF+JEdz3McSGuc2iVLHmeJGHa6TuPrU88cWcfIwjb5NkysRMIvhZ66ArhEm4UJDL6bCMcQ6PHVN75ubnjRVM++y9cr/cdZXgoZKnwlW8tQzQUGfkUnFhYGCZQm1lN3maQYNnP+Gs/DzH9yP5WvaaOOkNg/XNv/LLEvYSLWKk9OL+OCXb0Y0bKGY60cYTSJfGkMrKCJSKCHd04c2a13SOpPmwct619x0A/XOI27dKlsjRTgw+1hPA1VZ6lFlY07ZLK1P7yzyGnOJNYvnzmo40X2JrNF2ekhNytMw728q6nok9RTwZULPnm3jidR8DTrz8QM02EboyWHNfd9GcLyCfW/5HNJBTJukFQnxeOUYtrSn8UR3AX/x0Q/gvR/7azx77wtIVFKYq82ikKd9hkVcooJ8L30212wn15csGm5Y3ghGVd83830/RTmv8+NaHYymBCwYjNQPTtKGkekigTDrQYvwH7OUlgHPExf483QmYG47MTGpxc9eMOs4WXW6WtvkbjquF26iawoiAv8MOCTvV7hAIq4WXZXDC+0Welf1Y9Ur+vHsXS8g1kgikgWG1w7hvv97BP3DGSy0NqO3VNQzpCwLhc15zby28sIcuvUqKrNNLB7LIZPqRyRISXybJ6icnzhS5wYA+JyqlbptaJU/VMCgxI+lpmq9OcDKwDtiGDzpjW5AlFQTWgku1FCDIaneqFT+ewd60bOsoPtLjCKR5eB+KCPz+myIykwV5dkqZidm0W0Q/DSZ1zgoHMishOyziAzCtZ516pLRRz9gBlujD+oEk3KFUU3ZA1I7jrPCGnInRx4IYyHWvXwEyVwCv7zxYYyuqiAar+nAUvD0znyO8joztYh3f+ZbiKX7rL4mFyKWQ7JnJbrJAuLZAiKZNBLpHCIJU9mQwoWE+LtC4Bk0/PS7AN6E9bo9wKqSgJnToXWvC/2mtDrWC3QZUmrtnVMCzR4GFxTvQAFLv6y/JFKDyDCWzrB48b1TkhL0ZwlVGxeYIA0F6ViTVlmUR9rYcNM/o7VuFfa/5qPItQKxk7qxCO6fexG7oxVsCWtYfebZ+Nev/TsGz16LrffsQWe6g1jKUGJDeS0rsGsw5zfOufaV+k0e1G1mX8uLtkeXP9eK8emw/7zkFfNFOdhuQe5Uz5GR3TjAHCs0CiPfn5tX4Iy8ZiuiKdoQvtExfSrD96BAnI3HiVi6BOiJI622Bnu7bTGomMqSUdWNtHHGprXIroxg29070C1nEUsZCj20oYSHf/Y0cv0ziGWO61kxmPb09iKbzmjRzM7OmIl1bRELs9PolNtYPFFEMtqLbpAAurzOtE5go23SGI6v46RiHFAiJ8S2pbFKIU+b42UdZ+uLt8aGyPVcQDqsDYiE7BU71h6d51lmtMIGFluLKPZmMDw2gFRfCsX+IlL5JHJFyr8YZhHpRNCqAfOTZSzMlrG4WAWn7VqLvG/UvzJ1RD6QWo3WKXQ/NOcLtdt4vXSld2L46VwG0STQP9aH1ecNqwW3/cnDmDo5gdzAIR1ZrMoFIjmwVevfWZ1UG8DXvns7Xji6oEDRDRNID64BkgVE4hlEklnJ10Sp501AjJkWNyuzJ1JGZcPqZsV5rQQAHWnII/PKfk9s+P1Q5G9q87imtk4hl+Kq1nNpkicJeLjeCn3H63UHsf7ON3cMXl9fGrvE+KMaIXQSI0JOUVedSznWWrOF9de8HvnPvxc7r/0ickendaM4QHXf9D4NGdzTnkY0XcQ3PvY1jJ03hjWXnoVaO4bdjxxApBJHrEVU2VQVuJGpjMHTdXhoSKemUn1GOIdYE5klt5arq1JbVBptTCjr9Zlqvnn8iEXlfl8b1IEjmgoSPbKNSr0mLi1V/0I29Li4iJYWcmhUjV/MhyCvXFdfM/DZAo8gQo2neErvX+8wXSaS3EKWCov0xmnX0bd2GGsuLCFsdfD4T/c4+46I5GKDWBK5lUls/uUWjK2bA2LzOvXUVuDMaqVGvwCEHTuhpLjI0qfeQKOyiJ/8cgv+ZNOfIuykEYTkc9sAQUvSvIZxcNNVax41tyF1lgE8pSnnw40u2mHcZkltOsurXri5Zke24L3RhtCpbkP6BNx860snE0dFHQrMcoRrqFybRyIXYmT1AMbWjaBvpBfJBIfFI8JiVK86HTLZhEgVzEAv9r0F+vAanK+xDioYxbbdaOD5hw8gbMZkU3L05GGkSy+awFMkoplkG4K3TIIBlfz4Q4eO4Hs334VnDtQZwsUviCRLyJQG0QwyOmkTGQ5+5MWkYk+XG5Y6VAK5JMrIAKmIgxgzFr4SueKntUeDF9ddGeYyabUdZGTlFiWPa388nw4w+UFsq+GMZaTC34EB4ipTv8lNZ3he8hIBwZ2EJlRudXEzbFgPNuyiGQ0RGy7i7Nv+Dfu+/n9I3/GkHlol0sEDs/txMt7Br7uzaIQB/v1jX0dvzxC6yS4GVpew4iXjiGRJK4sDrSjCJk8HXorxO1WzO41nMbJ8K2JphNF1FEXP7qJdZ5pm6gmcYZWSvJArO8m9eBdBllq1jaBMd/MG5mcW6djp2kldDUb3FovKNDrOJoW9Py4Cj4h2OObogBciz/Qt6ka6ohISACr055HuzyKVjyDIdNCttrBt8x5M7KtiqKdfgYenMp9LMhtDelkCd//sAZz9stC0puQcaCVEX28vjh4+gBgBNPka2wLn14kjB/GVb92iAY8zlq3HZedfiuH+lRrcCEO2sKz25yYNWKN1CM5YSs+U2tzzbCZW7cMo2WZ+3paoadK1x4zAYJ2KU3JBasdKrMCsX4mae0cIBVN3UAiLWQI5+WfTV2q362h36+hwTakHamm3viJsxcSRpH1KlHW4PSNtPjG5KDnEv0dRyPShHdBDKI1Sfxbl9hGE8UOmONKwA4G1NF//FJ7BPv4ifnTrA7h/60nbuNEUooksOpEU4mwPpfOIJXNANI0wFkUik9WwPliOsDxJmCg781kebrId4FbzksgOXwr2jb8mZORh9OBp5E9IRk6fTnLj+pTR+LvuPjjqmT74aRxlGfY6Rgk9hITeOoTWvE5PQdsCHtp127QUCIuFmE408erHbkJ11xFMfvBfEWu2cDLWxmOLRzCR6OD29oxO6He96R14xXmvRiKSQSxIKlK2Ig0E8QCZXFILvo0W4im7uUbnNObREmLOWiYamjGx5nEtbbHxPa/9w5TqlEoGvWH4JURaEzG8f2l0YvTR5YJzkx3qJSt51vuKJ+3IzUorHbXN0HzdeaGd5plGlhlXVhP1Kqd/aqhNLWBxsoGTB+YR6SaRjtLhjqbSRYFC2ggdo0SeaNBs+RDa4aJOr76eXm0C2Xa0OavcUrbACO8VGRKpFF7ctR1f/96v5AgnlROWPd0Qf/eZD2J2ahbxsB8B8ohHc4jHUgKXCPYws+CJKlAwZJukJblVugOIEqna0thewh0o5ytDcvOrEndX/GS3Gdg7d/RO8aQjhgxLTldahqwJiXSzlWQIPrEYvk6jabPOtAzxd1aWrG7diePsABdDn03RhFx29li7aKGnj1NfZFIxbW5henEPXagta5CAuRt6d84XGnSwxjJuu+cJ3HTvHgfwkdGXQDeSQDeaQoqbN0GQLiOnSyLNiVxRzz1wptogW44ySdpfUQ3fc237+WhlxIdWXxUKgiZClzAdYZ2gblLDn7AexJH+r++XuBpSJAueRg6V9pFRQIqTqVEqtiTqxdVgabbQSKncGfBSjbYwv3IAZ97wJQzGsnj+jR9HqtXGweos9qKMnYk6HqjNoBW20Zsfwpc/8LfIxPvRbXQQxqzWjCdipmFEBQ2nB9QmQZ99uyXhdvrmGhjEyOz1kj3t0IgWdhLwzzwBTe7HNHB5UhCgoP8rTzI1z9VfNAQwlkgtSalSgzmItJHJxhBJnZJtYaYh4I3AXtuE7DRZFdCexCRRO23LaAxEsTpI0rJqZ5mNZ4qqGZx06obIkPUTi+BE/UEgUlZfUPYligbmEGAC7yYxRBK7mFnsgycS2PnsNnzj+7+wWVG3mXLZND7/6b8wDnWtrs/FINBX6Ee7TiQ2jk4zC3SziEeLrn4n+GVtQipJiG0V5Wlrk00Bec8aZOHUi9W7PKlZtrCmlqE4gdEEHQrpR2TXw3tPwzdNn7khA6G8zpuIa4oTPv5w4X3jdVsZQvle8+ONJ4nSG1bBHrOCClNsAVdRAxejATKFJOa7m4GIlXnqtWbTSv1tHt0sWYzV1ZY964nFDj7wxesRTWTUOgqjaWWBNghFz6AC4pkehPEUYsksujECVQES6SwLGGV3IYOGRNJDeRglSP10bUNlity41uqhKJshhNLuWSS7x3pnVsSbgrpa356f6Taxd7iTlKk0h4xkoO+zfhEiSpZSzKlBOjE5L7XJfq5DqKvxDpqXno2+T1yLwtgwDvzBZ5CaqeBQewEHIzXcWz2KZ2ki1m2qyf937/scVvasAuIpuQcqlWIrIEqxO474uTYWWwhSUDDgbH6e+kskHKSM8K6Nau0MEUm0qU3DyPvWaqjemTl7gomxxY1q6cUD9G/OrZ3pFEESD2bF4m5mmUikhgusD9jsniLmE120wXFj5lg7xtBFD1Aw0MlqlKlVOqkNyZ+hoF09mEYjtUsqItq0Lr3nHDQXkhhITZqLdRFo8H3psMeTv30cP/zZwzrx/cZljfeRv3qLpchNow6yDUIsQwqP0k2i/lIMC3OLiHTSaNS4+eJIJ0tIxqkYGbfgGjJQMEAJ8zeBcmY8HGSQjxNJElaOkAyi1pSzDeH7MtUnF1rMKUer1byqgpzxvokb0ErVNpMJ2BsKTJDKSiRxoCUxy9vRQYp/56ZN2iy0PWumI3XMdx93oJGVh0K83bPjuuHPk7TBzUfLzocefwb/+qPfoRkhVZHrikMaZHExFYsDHOiPctMWkMwVIUVutk5V8yYcvZHkHQY1m7xiNsQ9qq4PD8MD46/TIL2QPjfGxmjDWoZEAd40W6RWH3qlC5EWPHFen8XYUUuULOcd4/Sil5QTtJmdsJw2uU5p46BqwDroIv6ZazD01jdKxXD6+tsxd9N9mOlWcaRTwewlq/D9Bx5U/s9ToTeSw3Xv/yKyhT6kYvbw+H0pChCdcywtcn6lcOhoY6rR2Cek4DVrFvXPDNP1LSwf4bSxGk1kc3kbR+w0zb2BKWCEFhxMobgZSOE0tQKbG7RJmWj8FDPNNqoRMrQAOKSeiCuFVbsmlUaHYmeOyCL+ruOu8nc1OkfyhZwBTAlSp7Bn/rRbqCdeRLxQA8u709li1BLmRXHThkw7WUe5z2ttszbu+tVvcMf9z4mkwV3Az7tixSjeee0b1DZJxpm+2eepafiE7x+XM4Iye55gDHydDmamZ6V8yB47NyxlhlpNysxkEA2LCNjUDSOIhkl02taPVXbTNuEBS51toF4sK2czyu9z2oqGb5wgUtargX/7GTHf3IwvFwNPcUmcUpeM7TeXjrOeFHU3ABKphDZHPJ0QOMn1zM9WDXejHhxUIObr83kR+SXzjVRbOtAvOvBTfOlYBB/7xGcx3RlGNdqLWCSp+6PWFdefDAWIHrP2TiCMJHTopLJ5taH47/9fW+8BZmlVZf3vG+vWrRw6QneTBQYVHRUJOuo3I8YZFUEx66goKDkjsYkCDTRIFgUEkSAqCGIYdRQwIIIISu5cXTndujl8z2/tc273//985YPdXXXr3vc97zk7rL322gwDS+nnlIsSKhGx3yMOoeh3ZPcPtGKfojFqIjTtxgeusFlT04LguRL57dqO4kYP5AAvtTg8TghIDTPSBymoi3ARYPTIDtJBwVpSyK81bPlvr7KRF161aqtmuf4he+HTJ1u5UbMtzYrlv/RWu+0nj9jf141Zg4OTSNs+O+1jX3r/J6yne9AbYJgTaoifR9DCrwFrjaaRqHGaTMCDzDjAJmTZrZnUG4MH5uDJqMlwRbV5B1WElAcBPH5WLkFIcLYXG0rN99JXinxpVz9wiw56CuPGmTDq9y370Gcvv7iaJOyhaFjZeC71YlZUGaUlfrPSSvVhdFgyW7J654uW6wYN9snyQmlbXG9d18uhFN0XD5xwMYHYW3vHrT+wJ558SYYvigS8ad/X2Pvfe4B6jCnfSRAAY5HBA3pzgZd4PNJSxMakwqJL2mgNYCwJ0S7q/rlu0H4R9MFWkgmbnJgUXpFJ9zGhzVL1y/y6HwAAIABJREFUTrN6v9YE701JLZPuslKZweCUtEgZyGNTojDiacm7iQoU/QlHcEWXUqmiFjkw4FoNdpLz7om4cE3ZbEJiABrfyhC9dCepprVyz1ijWVSFgByYlBCvifH0PNsrEDJ8taaNT8zYcSeebOmOfivl97FmGvZTlzSaLQmZBcOPYcrK8xLxNJkhjfgx15/rsFy+X/zubDavWdHqFmVSvUYf+H+JDasObkUScyXMXIkhL6CV2FDBI0YChbsL/3ISfkr0NuUxyoucNyqGh6Q6PTSGu+FRG8OeXAmwrWEsQY2mpT+wvy0657P2l7cdaZkdBm3VDafZ4x/5mnWUKjbS0bTmx/axzlyPffP6222qxJhtl4x5/35vs4P23d/6csstkcxLJZ7jK/qbRN0CgyvkuKJ9qvGBHMebsrlf5TzhcHGt3AeHFMMFwUI5OShqmO7HnNoIuPB9Ne8HNQiXbM1aMsiPKD8C/NAEc0Jy583y+xpwFQAsKSHEBmtNf4jAjfNjVW/X2ru6RI5wLJG0SmvW8ssnrZ4oW7az03JJJ+YrjggjWAmXNWmC6QREDu2pp8z6Kdn13/q2vfTqhDY4HVx8ffKwD9juuy4R8KYG+UxabKRCaOogQvN72jbHKUZTrF+sKDh32HnpGuoVBPoQiuf9eN8yRAmVV7ps6+iYLVm0g6YRZixv1WpDOTSH1yxjzToN9DQ05ARMcV+kN/CfAXZoXRTIKu1jmH6UCEO0E5r6FWJrzErWevsGLJFCsYW8c8ES+VetXJ2wzs4eJ8dkMzq8rXRWDRuUGDu7GRA+oAFt1VLdjjvhRJuaXWAcgaV6d7VCcrElWlnhR0KXpS4CoEk3G4AUDQ3h8JIDE3FIi5zSXpdl8p3WkevU/bglotRllti86/taUR6k3fcY8gANuQ6eJ+Y7ejSxKyjU5QTgBEE15/N6o7MeHlY9jF5EfS+WUvBwEgoK7CbqWQtLu23lPRfYlnt+YYVLvi9v0H3fBbb1+4/Y1I8esblF3db48GtULx0vVOzKm+9WEg903pdJ2wfecZAI7r3di9TMvFBJ2pLh5daX77bezn4RCogGsGztHAkgJBIHQqnB64aAQR42x3owhwSkNBDUnEIXROB8spzrbkUxNRk9dSo54uvyr2EMpNDnbfNxMWSy3FJGCLNz9L2QB+sgU7pxZJBpBXwWXoxQvNwat6W7t0RwTyMrCkDHbCQJAzipXymPAMG6NWsVhbEwmmRLBTA27ao119q6DUi9Wps/fvYZx1omSU6cFmod66tKRwJSLCMdpFecNBLeNxArFH1BtkFzStMJ3BjyOjWuBG0yRWgQIrX2TStXSpYipUh3WXdvh02MT1mxVFDDAqEu6U5P92Kq0daRzlujlrZmnTIVOXbKki244DCmcqEkaNZqJK1Uqemw8nwi4T+XT6nubNkZa6TGLJllVnLShocHbW521lMjvDaeMzDdxMuGmVUq2ab1I3be6gvlQYnkrrxmrX3jkttsrJjzHBcvrlZqB7UQKEDhJEFKB91L3VLqnpfHTeIMldfCwmKfIn2TEVKf2LDy3Tq4nps55ByZIO4cnT0lVYmga8ufPDCmA0TPKog+kCviQ3PAJgh3ydM5isyXI4d1a0EYqDatvHjYdvjZ+bbwlxdt9PMXWa1W8gHXHz/ABj/+YXvmE0dbaZ9lVn3rjtaRzgps+P0fn7Cf/vbvEkFLJ1J26H8ebDsOdlulVrHRqSn7ya+fCMqLQqiUO+XSHfaFD/67dXUusVymV/cFcum9sRwkV6NQqCpUzw2Qiv/UJhM+psS5o4B+7oFwTmxqDoka3mWQ3EJXar6JfVZRUSQIb3DwvAljIFG2MFA7lekUKOb5l/NiNa6TcIuylXJgKBQVG5sesVvvW2uXrDlLlEHCdcA3RRNBJsbfO+TNQmKhpTI/CO/mHl9pS6Nql152nY1PzIu8oKjIzL76pcNt0ZI+AS3VMmNMaPwvWk9Pv0Jf1irqZeu9Ei40KNlWoopAOIH0QH4psC/pAgc+LdGnUYisH0j0GPt8vlOMNxmFMP2PAxJbM2nw6EOZpMUYWGRo8cQcCed7K3SnqQMZWqYaVOr20AO/s6mpiu20bDdbvnilZTJdajKYmhux10JvzBeF1itqKpdCAwkH0eVk4bk3NMKlYV3qKOMMEIWZrV59qW0am1KE9G/veJt94pOHCYD7yhm3WLHZa0lEBQC1WhlLZ7g+b5CnPV4TDpizVKPu7g39hEmIxXFWUmlem2yPn01sXHVwK7a/uXV2TxDDYB3S0J4WgSQXqHY1x1gmwkT7wXfBK6G57nv0ED3E9AXhSwghsXu5bvbZf7eBr33YRn/6Oyt84zuWalat1KhaK52x6V0HbOdrzrKnDznW0oe90cqD3knhIFHTrrzxThtfQFKlZZ2plh313x+3cmneRka22s8f+7vVSGCouQUADkNy9Gc+ZP0D/SpBqLUrge4zfOOSUNcowQqIA7qraXoJDh3IZNpaVY/5+X42xxBqJ65kssiXcvhZP8JuR4Ep6WgtABViCCxEPkjdaJVcA8tbCYPUjvS4XNpFggPNhm3ZvMme/efzVmnVbLbARPWmGFYnnXGMLVm21IaGBnWdAvqkEBEGlyn4cjCwUa/I4HCASWXaoEerYasvuMLGJuYUVcgAJxK25pJvmCUrVipWrFIuquXP1RvrXquVfKQ/b0UW8V5DtSK+fyy7qQElGEepVgRsRfcYSl/CAEI0wH2o9Bb0uXU4SUPCVADQZxEUQq0YOVRE40HUWXOEzhFWoL570YVX2eZN04YIP4CVcI1Wy978pjfaRw55V1t0XDKv9arQZxBjUiL0onxNMCTegJJN422rNjszZxdfdoPqtRiQq9eusc7OjD366ON2y3e+bTa4r5XTSy2R7LSmDqU3FERD53xlBUHWEM8Aznc4i4jo06sF15oDzjVv3uk9LZgtCmEDDUBaSm01gqDIGObCbl/XBVSIobSTWNw7RQ6o8rSgNuBaVds2CWB183W72ZKLv2z1xXlbf8r11nr4cWuiHs7JBNxKJm2yp2W73LPGfn/lWut+80orUzMLnkSDnusNu3jtbVZRIGe21y7L7D/etp+V5mbs4f/9q03ME9pGzVqTNTv9a5+1VtMbDBQ5AAjkctJIjhxnvBQHUOUX1au91KB8jUhB+TxgCG16jvyyMVmfSLrHKLCJhJsjiwrpQU7ca9gCIeH/8vfQOkk47fvVDzC9uL5RWlarLNjzL75sv/7V0wq5sEllapbNlh1x5BH2uje8wRotn0b3///yFkG8d0rv44d32yRB1iGZaNk3zrrYpmeckM+9otB54XnHqwcVcKi/t8d7mBvetxrr/qrZB5X+uCElBk/Yx9wjPLV4uH5YolfTBIJQEhPfuwpiT4Tns4UiCBijvIijRDIHNWzX8Mqonu31bmicTsaQvG8I4zHMZ5xxkVUqAFYJNcNw+EGM/+tD77bXv34n6+vp13NCk8taSOs6FRUGkz6bZ0GRJtT3wQF434VCyZ57caM9/ue/2gc/+J/2tgPeaplswi688Ju2dWSzdaQ6rdq1yuazK6ya7vNGnGDoVM1JYLS9RIaFVfOKhOadtAPSzIZRmEz0tGW397dU2lGZxEO6qObHxtIhbHioHBdN7p3NEaQ6faO41i7lH9BILaAGbLUsn0haIVUXwpy1rI0N523n606x1I6DNvO3F+wfXzrfBsoJ6yDcTDlaizebt7LNZLO26q4z7YU//84qNc93/OFnFK7NzEzYP9aN2b0P/14PIJNs2pGfOcxymbr99ann7HdPQ1NzwEglK0valz9zqK1aOqAGb5DcwcEh3Tebzw9MnLVLmQrShiPpURfa4xsvX4kwobEbnrtiqWmfYwOCYMuC8qlhc8awLzZpyHNrTKWLmwnND03aMUWJ10bP6sYN6+znD/9eD1Oc2kbLyvWavf9D/2n/9q53tsPKWBVo52J054SculGc87qr5uY4SAcVMZlu2WmnXGAzHNwUYFXN9nnta+zzn/1ooDnWhAADRnHQi0VvZ9REwoWFNuIdUXBeV6b3NsizAA5JjzuE5tG4xDq5YyUOXqkc1nA5XJEnQsqFkwF0WrR4kXdKpTM2NzdrOcpDon0CInUoraEWy570mnenAKTTTrkwpC2OHWBkcQDHn3iEDQzkBGIymRGVDQxbjJTm52a0p1XHD/wDFxwEXUcDu2StTIdSld1228tq9YqcwAknnGLJRsu6u1E3SdlcJWkL2QFrDPyLNRLeiy0pJbfVIqwANMpwJiCw8HlEE+TB7ky0h0Zf85/AAG04P6KlEagSmpbyZBzrIxJGQD2jNZP8SMo3Pkajo9qyUqppKRQsyM2olQ50Wd+h/8c6Pv52a+Sy1nh+nf35xDXWu2HaOgiRMklJ1TToP1T9sGXVZMPG/nWJ1d/zWsnAuEay1495oFwrG4b2tkd++yd74rn1eigrhnvs0P/8d2tWq/ade/9HCvCx3xVA4F0HvtH23nUHW7FyRXuwFpZfPbsingfeqiyrh/o+jdDXKW5MdVKJk+tKDIpZAlPLJ+wBvhASbScuH9IQFp+NHME68jDE5eSJ4yC1MHlBZQc1MSRt8+aN9qN7HxaAwUEEZClWy/aGN7/JPvOFz7cxBO2D0Jboid82AKgyP2OVYqFN4eW6kbKZm5+y1eeusVIZTB5/nrKDDnqzvffgg5yjWy5Zd75L9++dVC0bGxsTe4swlwNIIwYGNWppd1ALRe0j2+GkmJD/ekNBRgeK94pfhPBKDXgeQWhBIX/CVEJiMBpjVYRIB9aXk/Pxslmxqij7eT856VTDyRnNhgQWzjvnCgdnE16S8464uq0+/1SrVGbV0IEoHNMPCaHFvZc6p0eXfG7/4IDNzxeUg09Nzcgrwo5Dfobcvb9vUPf76KOP2YMPPiIwFRwFeqeUK5Mm9tTXTz3Nnnl+zH7+u2etmuxRyZP7zFLfFo+acBlHiJF2aqpKhOyxrXt8UG42InyxHuetWWF2DhBjyMFizushoqOf8soa7NywCt4tlbfGULelX7eTdb/3QOveb2+rZxNWL8zbyJ+ets1X32d9r45Zg+6UVMsytTDs2qOENkd6pitplSMOtHKiYnXxNgHQOLx+XRC6YymHDpNLrvq2lZuEl2Zf/eInLNtYsO/e80uroiKhPl0ecMpWLem1zx7+YXV0KB8MaLKoiiGP8dw9KCuQW4mM79ROHz/p+Q7ibz7Eyr0qG9jZWA68ONjgTQmx3hdTCT+4/uVGMciqBE8QsYE445Ue2OnpMbvz9nusWfPaYZl5Qo2aLVu1wo478QTPo8OwMJDbOJ+Jkgj1ZeiD9QpNEOTyPlyK1/f09Nr4xIgf3FLTWkmogg372Mc+bG964x5+YDS20g/cyMiILVmyqL1+3HdsPyMHjjREMmuRIljj4DW3XwcOffTWREDkjJHKiPeNzkFSMmGWkFjeQWxO5TFAPRUBhNK01TKIIiCqCJgSaSNvxxx9ZqjJO0OKEg+G+vQzjrUEWEeSCAK1EPSrnRG3bcZuRc+X+49RhI82wYgmbL4wKwB02bKVVpgv2SWXfFPItvSypOjZtIVGRVHCRz7yETvgwP2UBnEQy7Wm/fXFMXv06Y326pY5a7Xy8rKNZMPBMHXree1ZSP6WPT6g+6UpQPUkTS5rqd0IF69NhwIFAARehTfBK6FG0D9opXzScsO9lt53b0vvu7P1vWE3a0JHROkBAGTrlI3+5Vl74eYf2cCWCUvXmpbBgoiUHtkgnuxHaZLYjTT5nl1t+rWDCr9J2Fl8wrLYi6m+23TW5/dIkydpN996p+2//wG2bLjPuvId9sivfmMvbZxTWx4sp0SyaR2plJ175jHKVfEO1PrQMJYqY8aBoFhjxkPIy6sjxkGVTJDWRLMpJ3kWz1lbLZeEAQkFuo/AHd7AvbUr9XMgvfHCQzXPD32wlw4j9cFORxwhDhB68/1KdcFSiQ77/f8+Zk8/8fcAfDWsSG0y32GXXHZpmDcTR4iGubNBwRLomzzXieh1q5aKYqoRTUDIGBndYFeuudWKiLgHIbavHvkZ6+/zaQYeaTCipNump6Y0FnN8fMyFC8JYFU+pXF1C9yvlCTfGiA9EA+b32Gld+bzNzsy6sEGpqCYPfhaNIx5GgntCrr27yc27A1QKH5NoeJUsq95hNrP/DmGlS/Y2rb9/wDZvHbXV513Vlqd1XnvWVq1Ybp/93OHaG5AcYrmLkBnecFWySt5LrnUI/bdxSh+lrpjrM2iMa5iZXrDrvnWzJZNZGUX6zXlNVbX3nJ122slq+O/tdVGFqenxtjh6odK0YqVp9/3qeXt+S9GmFlrWQjkDZU6xv+qWGNnjgy1CMMJJVIYWmg1LQ+1LmJV6MpZfscRSb9jd8rvvaLmVSyw52G/Jzow1QOUysEV8kjj/y82WbeOTz9qGX/zWEk9vsNx0yTLFqjXSZpk6OXQ9dAGR7AddWno7s3SZBMoknpuSSm/Wip95k82kK9JdwjPyoFm8uQLMGTaBWXffgA6Kt5Wh0le0cpWQrttKxYL9+S9/sz8/s6mtbkC4lkulbPU5xznNkFJFBklOZzl10zNbZtSHz3SN+SchICEX5Q/Kz4R3YgIVGG7sWldcKCwf6S2HDhYMDRzwKFmjRosgi+LSrp6zcCgoNThzykN195z00GZF0MhSOrOUbR0Zsx/cfo8sOb9XrbZsslywK69eK/pjDOXFtQ3IcIUh0uWSIgcpKyh3Z/zGgkLCeq1iU9NjdsXl31EDg2eZSTv55CMtnXZ1TAAfNQJIZM37ZQuFBa3bkkWLdI08lwLicFLmN+Xh8sahCYBDENVBkEzlIGfDNEKEyksLBT1jhrSNEoYDOIn5tU0TTOURFDxqNevt65PHJiVD4havqq7aIDKPfI5SmUbTXl6/3m6+8S4dZmq3KgV2dNiH/+sDtudeu8i4w8FWGsOYmS5C4cmQLjniLYMRokz2zczsjOfBoU2UfURU9sjDv7G/Pvl3HUxNWgy6VGTNr33d3nbwe95l9TrGpsN2WL7cJiemvZEeIK9WtGwiq8aCucKs1ROdNjLWtJ//+Vl7ZbRu89Zjicm7H2hl+rots+OwZXbocxK0OvcJo5qWZLQDOlOlqhUnZqw4PmGFZ1+16rqtNr9ui1Vf2GT5essyADpYA3GAE+qrTVVduUI8ZCB1SbHAYnIKV8yXQQHdUnqiPtOTsspn32YLncyLQYXR66hsHhXwo8wLaHjKNWdzHZ3KK5B5RWVidOuIVYolW795iz34iydDkd+nHCQaLfvmxWfoUPK7CwvzwSPkdIidoOJhr8TQOVzBa3Ko0VjicIjHvb3MrIZGeV0T1DSyn7hXCbABPqElHco11DhjmByBKZHVU7mgtJgXM4rrUSN6kvpx1qbGp+zG625p85OrlYZNFgt23U3Xa21iGCe5sEACATBsVEGSg/QJoTlaX+UFKxYWlMNNz4zZVVfe5m12ut+UnXHmcd4QENacziLWgC8iFbwjBg0pHQ4sX52dNEl4VEHLJlEN3pZD4ioZfvDcM7fkwbhvgUWZtA42/8ZYi0KriY7uob1P12ca43HRv8bgOSHfQVS6wHg23jCDyob3mj/x1JN2//2/CGqWPpWQ8P70U08ytlK9XtHBJWTnQzNpIqKsTU5NKoUSSxA0GK/ZRe5e9AaRQOGN0xtY/8suuVa8AOZE8QBJigTCZdJ23PFfs3QGz+nenCiCz5EKB6owRHFBuB5RORDnUrloOaLBWkrhf2Ju3dOtRKFszfmyFbaO2PzzG2z2n+utsnGTNcamLQ90XvN2JuW8tGSFso/mnQSqIIOs1QGDtwn0t9gGFSelCUmNyhPqg3RVBcKiTpC1tNnL6ZrdWt9k//3lj1oyBz+1oBwml3cAJDJusGoKM7p7dCDiYGEeNCijxHGaTXv2uX/YAw//2SoisGdU68tlknbc146wFSuWtjVx2QnaJELWyUfTVizhdX0mTSQ16MDCOop6VMGbxFolHgwAAtlOVSbaA5uh3/nnx+kKeE8JxakU41PpIRiwebhXjd4gfWm1rI+pgPB+az6i8/qrr7VEM2nZdE6o6VRx3q656QZvRQylJZL9tnEMqDYHq1YpSeGhiQepl2xiYtx6u/M2OrbVrrry1qDVxBpk7JjjviSkXrV9zQRyCiiHj9p2rL2io8XGXLJkiU1MTbjxDqJt5K2E0vLAGimSF/WP+wYU09CtZErfx3vG0lKt7lMN+Wx6a9nc1Mw70WzSHF6vZPjfnf/b3d3lhieTViSmAW8yFFn74X0/tl//+n8dmMphBLxF89zVJ2ssCXk841kgzfC7maR3xnnpzjW2eXZ9vd02NTWlZ0sEpucnkgwRUNNefHGD3X3Xj+VICO9pKPAGiabtuc9u9vGPHyrwy1NPP08Ab3FWcmSjOcbhyqS+5kgCe5SSeG6PtwsKVfse6ozUEUVXdM8oUCGIyIlYEb6ilKWHZZENtY18gcV2fSHPdfiSWnxoKxOoxWGSQkHT5rIp+21y2h7LVNV1ctzXP23lwoxyP5DCyelpdYSwwdkkbHDQxu31o8i5uCnQTz5306ZNCqXuue9X9uK6rQpRIXV3pBP2mcMPsX/919fJikt8K1Abe7p7tOHkeekU1fDk7YTBlB46M0oWMqhO8Dr/ooxCCcOHNbdVNxDOzuVUQBe3JzBj4uKomSMYxO4er5UK4Q80SgwDh1bheXHB7rj1eza6ecxy2bzyp9ly0a6++QYrl/zBik4phNytOmR4WX7CZO6rUra56Rkb6u+2mekJEU82btxs1157m8+HSpjE3b961OfE12G9o4ER2URytH6v8kKI/pUrAvyQ5CFHdxpnwuhKwqty3RxSIeSphO200yob2bpVLLA4VMw1rb03Soqhkjjy0ZzbaKo+xlPU1bBm8IsLCz5cnIHogHA77rijQl0OELjNjTfcbM8++091FZGeYYzz+R47+9wT5Ol0LyIh4bmzNjc14cZCpT0veymCiXTe0LvuP3fmE3nyfff81Na9ujk0X8AdcGNKmnH8ScdIXkh2MJwnnlds1pCoXWjMiHs7dq1JXIEvDu7fd3l7S1aFsC/U9IDO1U8r+UpnSMnbhhm4PhOU/CUucuhOidKRQdlBnxFqwRqiFUTW+D7vV0iYbUxV7c82axtyLWuB8taqNl8u25v22MkOfPt+uiHCRQgQ3CAT75jAjuedmpy0TsoMCcJaNk2XvFFvLzKkjNPskKLjn578h11z/d0CJeh3xOO+86C32CGH/Jdeo4bqQCBwEAjrTtO3o67Sygo1bl8PBxpUXwxsp8ikicin5sCGecB8hq83qDRtW2HMYmjUj6FtDGtl4cXEIkzyMN1HZjiSzAb+1c9+YX/+wxPSLyY8nq+V7AtfPcL23nufYFSo/XmPq64tWHYRSAANaxWrV2rWrKF1PKcG/C1bR+3SS66VvCpe/i1v2c8Ofu/bVbNeWCjKiGZTaZuemRGxnnv0JndXT6SWyWu6uvOKFiIqTq6D2J4a+ANnm9fxO/wuh0jN6LxPB7N4UbtwkbyYctAJDnjFmvhasx5+cJU/57tEOxSpRs7AmzHUxighw7RdftkVMk6u1AEWkbRlS3ewI7/+Oe0Xyb2GUidhf7JJia7Te8nTSf3J/YpNTg7c0+1lsXAu8p3dViov2FVrblTLIt6fL5whTm+XXXaxQw77EPRkPQNO1PaOh3uSgQ57UVUGxoeKiaeub/f+mOAnV+wvBQyNDNmuTqlDGw5mRNO0ELh39ROzeg7wYVFSWB+K62yMhtecKImQm/Lgs8m0zTYqVutIWWrVYivsucieWZixB37/uKwPYIFarMIcWcCco796uA4PIbl3eqRs6bJlsv6O/BGqzCssZTMPLxpqgyIgeXScIEX6ysYNdu7qa62JymDSB2qtXLXcTj7xCOtI5iybY+yDK1q4z0zooWB1NOM1rIUsv8Izn1zo9V1XamANfZN5eAXgw0NwZNkR8RgWubfmMHmOGz1tO3pRLdhJJuoECaqP4q4GttfLL71sd91xr6WYUl5vWalet30POtA+efgn2yUUNTyEkp6Xspz9QxkOnrLVncIIQLJ164jNTM/bNWtv8vJW0+wrR33ZBob6LUekEuIJs5r6pNUvqwPheeXM7JyQ20gsiQO4AXySrIU2IdEAtVWXtVUzvlKUvA5ftiNjC0Fz2mv52wZno52t5pagEaWy5XaypdK7Ar+AaqoSl6tYoMpJOMuzuvTSK2xkZNQVP+T10/aW/d5oH/3oh937yXt75KNUp4bCSF4RF3I/7DkcCRRNwtply5bbxo2uQ6W5SY2Kbdo4bnffdb91dOa1z7jGBdDyjk779KcOs/7hPpdI6uiwhdkZvYb1Y9+7MD8sDJ/J7KIPoSQLkh0ObfvgeumD2l0gGQQ5mfbBDQQAWQNCXWlMIS3kaLQCZaRbRHxvWj3RsGZ3hw5poydrXTsu1t+ruy62Yp4e06QtTM9ZpVy323/8U1kVeMOIVZMPiNFUqdgXP3+IDfR2WblGWJyQFacPE4V58kg2zfTMhKw23+/M5W10dLQ9e2bz5k120IFvs5nCjJ1x5hqbmCyo3MB9dHXn7MLVp1pvvkfavpoWD8ocvK3fO0iqN1XH/IwHyn+RqhgPrkJdqX94Ez3kBCeLeHPCtoPrDClZ0TAwTQIFgeIWYiEPP4M4t09m93wsHtz5uQW77JI1AlDUcNBoWe+yxXbGmWfrWtVmp3JJLEU5G00IbzphCzNTVizMyIsNDw9pzX7/u8ftlpvv1OGrNZt27upzLNvhhzaWSBhDRxrQle+yufnZdhrEYY8jVLlGNjyhJZUEvDkGItFsiNwwPT2jZ0Zk5GQJb6cEwALRlv5ZKMl5bTuMlgxhMT+L6UA0hrl8t68nayREPtS5ywBOXgM+66zzbG6WecKu48R6nHTy8bbNwWmqAAAgAElEQVTHbjvb2PiYT2+kbioEuGEtkPhwPaXinMpy3NPs9JRyV6538+bNiuqUE2dS9u2bb7NyyaRdRaQoDKBRs4HBAfvCFz6pzq/ubk+FIndcVYWg8SZCShFcB/qnt4xGFpw0wMKA7sSTK/d35hT/C7pRgme2G5YVaV78EuPsherKEzSsmEtasi9vM4MZm+1MWKMvZ4munKV7UCQEmnc3T7jXSieso5W0JkwUelvmS/abR/9s6zZPhPpgr1WqrrqByv5++/2LHfDmfUUOTwf4HlTW5VOj+FjgkKYResuKuQNwwGKA6BFi1Vslu/CSG+yFFzaKLcRCQB6/5MLTESG0RDpq/3rYFVMBGRKQbMm8OpLpBBXnJgtICdPzZP2V6/ng6HSH82SVF0ZBdhD3KNcjHV5y3RD+BtJ6BCZ8j9Jp40oeYglJRdEbJiDqX/7NK9XBIpwgkTJY2ZddtbZdP465UvTokigNk80b1bL0lCdGt9pAf78Oyy9+8Su7796HZEQofFxw4WobHO63uXkH3Pj9DjWsu+ffOjqqTQuvl3VgPRjclksnbX7ePTAhfnFuzhqAKxna4jyEZeojXkXjV6gpKyUCw/DSGOuIlxUoKgka9lAct+kgl7P5/J6kl0bomWH2jk9713NGUUTPqmDnnH2+Vcre9+yAUtouu/xiGRfRDquw8ZjMkFMoXFVJ0D17MuGcZb4Qkfd+aq+5x9IXf7/xhu9IUL6js1v7gSiO/fXJT33ChgZICXx+kaobNKyEFEZaz6HfV6qkgVYcS4UukO8OUljNn1btTzFGVrWaBJpPqkgvACKMOaynTPKoGbxfZ8LSOw5bZcWAVXqYMNC0Enlp0JnFIuFBgemxQjQnk89I+yfwnRU+ohvVqNvk5JT95IHfWJ2ByTnGUThyCsCUyrTsy/99uAAgWtpU9gHgSbvYF1azo8NHHPKzwWFU+BMmnWg2BS1lTXpgG/bkX5+ya2+8y8OrdEpDmc5ffaZlMjWf7RsOXDLrVEIeOkwlQvToIWUs2sOsIdlT6vASyPZfHiIH30mdMhA2hH6HAeGANF0AY9IiJszzsJqNKHazcno2Laiq52SIrZFSeD9x07598y326qsbVQeVbEAyYZdec3V7M/D4I5LP1cQcmmiJjQzIt3nDK1ZamNdY0J8++HP76UO/0rNHB+rKtWsFVM7Ozckjo1jB78SRK+R3ceNFD0hqUi/7QVe/q5kMqBpCirOiHgqdpuUTAQMqDYp2+Dc9q573aW5wkGfNh1nBUs9QJxGlFUgyPgiN92Y/aDhYGPzm+sxuhAnrp6dn7dxzz3ckmoMIut+RtYsuOl9MOxpNpECCXnMBbe2MJH6IxNi/1JcVNaEXXXO6LV/sryg88be//dN+8chvJHkjrx+ihaHBXvvoYR+wTqIXqZsglMeM3EhqaVl3l3tz4R3pjMJm1fzDJM34HCNnPvHHnd7cwtPy0DPNhC1Y3aqZhFUHOq1/r50ttWzQios6bKZZM+vqsJRKCPhLn/ZO6xGAUnFmTjfCDBUAGG6SBwBXlUXhQuK0MR2erIeCExMT9rv/fcKm50loIIZ3akwI1rhaL9tZZxxv1qhYoeggCP8pf8h3yqry/s4VLdvKVTvpYKmpXZPbQCPr0oJCauTo486S5ebmUfM/7ZTjbcnifpVFWEwsp5DYdNqe/+fztu8b/lVhqELHunNWI7I+PTOt2T+AYpE2mZVkTigBCb111g6GUGUwjXRxcEHzlkLfJz+LpAQeFrVr79bi4MY8mfAOPSQUIFnPhP3pj3+xe+75odg+tIpRq117443tvBlvHRk98br0WVnXqtq8ZbO8R193p8Cq226/yx7/w5P6/XRnxk465RRFMOwN6qHkwXEEJmvERoNGOTMza3vusYfPBgboq1VEzKDEQTPDYL+TZGCW8ewJOVkqjBesN6K7GBoDAsE+Ep4SZtDyORFoEodZHGSK+97dJcE5rpnwVwbXx5FieNl35KCFhaKdfsZZDsIS6WQyttPOq+yYY76mKIz8ER0pDNj4OBEg+6aivcs9VUpFb2EEoKOVr1jUGm4fyn/rmpusXKyLp43KhWZEJZP20UM+YCtXLRWSrxwWOR3uLxBvyHdhyEUBOtdjdsCP/aIDLCDO8ReF0D//xCEtDqmhDtiXs3R3p7WyKUH7XT3dWox0i1EIiGjCrmqoN1HaRaG/dH52ToyoqExIo7dCmHTa8l3dbe+NvjEbnwslb9V8n0TCRrZM2e9+/5RALjGOArm8VK7Y2w58k711v9fpYLF5RLKoVq2/H7JI2nKdPfJaGJHFixZ7eNZqKnf76xN/sl123lldSRzcY084x8pIodJHm8nY+973H/aB9x3c9m4sipBO6o5SE3QtJaGjgafsltZDajYbQnGxtxS0efsDIotMbTvwmmWwwgQ1IdUB3o80Ov1uQPCrNe+KifmNpD3xEhm0f/PWnc/bhvWbhZSqFlqpaDzIFdddGxQPGS7shiSGlfF6+O7gwKA8VKVcsPmZadu4Yb3dccf3VYME61i0dLGdedaZAlbmCgVDXoaNxf3iDWP0gAfmGivhcPmwNUf0ObxEFYipwWQDvOEZahpElDYys6WLh0SiIMWhTMSG17jJYPw9WnMRPkJuIiRI/YpaNMDc95rTTltieLH5yUHZXzxH+mVPPe0M77flNR05e8c7/s0+8MH3e5seTQjzc0oFXC8Mj1uRMdLhpSxYKstg4JW5Z54/pSUiBwz5zTd9zzoynS5HKxS8rNz2S1883OqNsgw468PaCMRUq6x7Zp4vh5k1rtBRFSYVOlaRUmqnUme4hsTdV50gVDnmWq6P7GR6nwgeWDRhrqjC0DBqMlLAiO2xevwZ65E6BNKHNRsaGvJJbqGJXu6e0LzKFPaWHvAjj/zOKlXCVAJF16SqVetCHo86+tPWCrNyya+XLFtm1RrT2wGuvM7a09trvb0Dbs3xbI2GPfDAA/aOtx1oiRY6S027/Kqr7U9/edYyGebpJuwtb36TffmI/3a1ytD8r4I5qJ7a9OLwMsZpOgMGSwuQoCl1msCHd2H+q5MouG4HojwfkuVvxfIPyGWwoGrf2zbdnVBRHTTybhkh4gJhNNoyFMI1tCorgkAuD/GkaeecdV7IP/01qy+71PqHBkNrpQOlMe/2afF1MaW4xl133VVtkYBGk6Njdvmaq2z9xhFFJa/Za0/74hFf8p7QdFoHi+aBXKeP3fBD5uioDkJob4zElMgG0kFGqI/QmQYOt2xG+BtLTGAlDgjVrYqGV5D4ZSN3d3XJ6GYyQe5Xapo+j2lsfNzXDGYZ1Cf1EGMQzdcII0FzQb5bA9fOOWe1vJy8cCppRx51pDrEmF5I9MM1k8viff05IgnQtMIsA+U6bWZmRocMCdresM+Q16GL6re/edQe/+MTCnmlJ8UggEbNPv3pw2zvvXe16WmQeL4f21aJHreN/4yht3L60EEmkC6kEBhOTZlkgDhVi/uuObkVw1qFs6F1T4AMlEAU9rarAUoJPygS8HssUHTnvG5qckoW0KmECzYwNKRifDzQcVwjUphefmlpmNWr6zbbU0+jLuiWqMyhltSF2XEnfjGoaTi6uXjJUt00KoPk1gIzmi3r6xvUweUQR34s+QjhWrVcst/+/jH7zq3f10hHCuWrVq2y8847r93gz/06Z5q65YKsMNQ28qVysabQT8oP9Zo2sTYh4Av86HLRXnrhBVuxYoUsJyGfT1v3QrsAIrE6nSmjNY1lJrxPoiUghTxLXGV5fS/bOLnDSzTpVDYwqqB55u3Ms86xwpzLw/J12nnn2bIdd0Beyz9bAE4YKRkIIXgtrpEQdGCwVyDMb375P/bjHz9gY5N0ppj9x3vebfsfdID1glXMzwvlx7suX77UXn31lYAB4G3CoLVQ22ctZLBoZaPHN5SveM+a6Kt1l5RVe1/Nli6lvFfQurPmZSbC5xgxilF34CmrAV0enemrCXhZsE7V2hvyiqD/aooP9whyK+yDWbSJpD366B/s7nt+qGgBh0LIf+FFF3o6orDa07CFwoznrgCkC3xG1hbmZ6xRcafE/TJOBoWVQamNgOmYXXftjUL2yaupS6tslO2wo4/9iiRtOSORLgu7bHx8XPtGHPcAlnluD+rskR4YgqRZG6RSOT0v31tpS/zoutP0xHWKQ7VOmyBMPI8oq48/SFilVG43F7NIGkhNrYr2JkTWVOf0dii+D9sp6i3zQDSqEgHrvC+oUFRr2dxC1X7y40esWk04Yi3yPCFVy17/hl3tfe87WA9d6KqEV6HI9Vg6l9UNUg4CyYtJPIsDQV2zS8slhV8s1rHHneyT0TNJhTHXXHOdX0NonueAsHj851I7XjZotpLKQ0UwVygPcJBRzy8US01xD/kQy6cWuJCLcX/R+6YgNwSryibyzQkguC3MjkCPb0Lvc63VaMfjetzjduTz4rR+85uX2+io0+94/eeOOMLecsD+Mn7xMPtu3/ZvnmE8uJVq0cZHtqgDa82Va21yqiCvdPSxR1tPX6/kQjl8REwYLs05azo7jY3mU/x8OgCRi9ZfIuRueGK4qrpk3YXLBZIlUzrAgGQ8b9YYY4j353mR/ij6C/OdQKNBnXm9lESCogp1eQ4uho9n7FGiYyUut+vo8f0//In94pe/DtMinGNww403WKm4IGE9ACmuNYoDaO01+QJJ26rVSs5LJoxm5pK8ovp6MTglu/ZbN1pWoXnQA6vV7BOfPFy5LXVfnS9IS7wnTADx1h3gigYpEjA8vHf6J9zmeLAdJA2i6D/81knbBNFbXjNTzlKtiazvVoa6GjWlpC3Mz7fRZiycgw5Nq4fWJiXRKbR0nUYoRJnp9Wj+hG4QaQdlUQsoaaI7N481ee655+yfL4xatZ7UhqEvMiJrR5/wFRXHKahTKlWfpoj+PCSGNBesu7dHh8sHOIdZP5aw/r4+bRYOwKc++XmrI8Kd8qL5TTfdFBbc5wBB/YtKA3h9X1lQR5hAgdlS9fxTOUk6pfyGdYNcHz2OvEoYiAaY52UD6rEgvY4WIs7m5Y5Y4nEv497ZzSgally3jEmt5DlzKmX9fUOSaHnqqafse7ffpWfDfwe881126KcO176OdNNISfWb8UNMGAioRJfQxNiIjW3dYt/97l02O1dUnffiSy9VZ4/wCKaz5/PKAbu62JxJ/RvyC+5ZXOq+PkVnkDMkSBBCZ1B5rrcQFDK4K6UjQbxBjQW0iBKtTU2FpoqEDQ0O2uT4RDst6+/vtSnVT71dDwNOvk00ghGgzZBGh8hdJtyV5yIlq1TtqquusY1btjgwxXiXzk67+OKL5QyY1xv7XKVlVnP6Y2fe97eoljVaKoOkU0itYh5//w9/ZOvXb3ZkO6DW+a6sfemLX7Levm7tEcn9CE12MM0bKraNo+G5eoupH9QIAkr5cTuGYvx54t6rT1So7EOjfAHFvcz5MGtHvJj76pYB3Vt+zmHmAfBhqqSQPwmZTSuUxDrr9UFMjAWkQO+slIoOC2WGnm7mzXpozWu+e+u9VqxQLvIcG5Qaa330cUdaR44aoHsyPodwiNwTj0sNjIkEg4OUn6DN+dgJXouxIc/m67zzLrBn//GKroND/oMf/EDXIoApCJe7JU0qf5a1C6oDHFxnS7EYgSBOe5tANi8NcB9x3WL+F8svbsx8IoTYVCHfUXmMhxoeGmkKX3pg8pQujIekajy4IMmICuB9Vp9LyOcHvX/xMvvG+ef67wcOefTwsV4vDrCZjY2N6v0mx7aIVLB27Y1Wrbm863nnn2/1pkcVsSdWWEgKI0uI1yHWFsZbpUTyQ6YFhFDYm098IBpeyimOHp6LeBGUMMnbMAYYAg4/h1czk8MIEQ938eaO+rqQvKOrGhpGDbhSUV1YDKka2ljz4qjznnGvnHLy6TZD6EnbZSplb/zXN9rhHz9cCPb8grdoclgKc3PtqQmkPzwbPc+sWq30rJUDlwDQEAJs2IUXXaLuNEeJHbR898H/x/bYYw/dWxh0IgfmIvnOVch1ODqtMlgoHUXHyWeKeRV42yoTxUkW4AA/vv40HVwv1nuNy7WCUGrfNjdIag4wi/CaGmhNw3E1CHr7DF2Va5Ipm5mb1aLNzc956EKY1dfbbufiQM3OM8LBgSRR/SgJ1Gr26ONP2LoNE1YLTfuiM5rZ/ge91d75rrcp+S9XFrRZevv6pWkVwwfCiojETk5O2tDQsCiOcDCx+Ljq559/xdZec5OzojJpO/PMM+0t+71V5QG1DYa8kzXx8ZGOMjt44iwf3q9dZhHAFLS6aPRG/IyJ8YwuDeTzapm82FvL0uHgAn6p40gHFAzUmzH0uRTbA9E/Ug3lNYPkKb9TZJJ809Uy2ZTcj9Q3Mx122dVX/X/qqzwvv+4QliXJp3P2wgsvyivNTI/bKy+9YNde+23xfTvyHXbOOeeoIcKHbfuoTJ4/B5c/RdmbR6DAPB1ijnC1IoMtFDuUv8AHCGWjvE3M310s1nNwiBaRaIBnivxdZiupdVIhposbaFIC/HKh0i6orxnFjYbKiKw/xgQnETuv4CMce+wJqihoHEjC7Jijj7HXv/71Mi5TM5MiXajxo8kAbHdUHNyobKIeayKnYtkG+7q0z0g5Nm3YaDffdIt15XtEBfY6f8OOO/5oH5fZpPfcjS+/42lZMHA5Fw2IXnR7YEoOY7upltsaDvyeEw/edLom0vNUeWgcRh5SpeYgFDdBmMvq4WFBxxYtWuzspECtw1I6WuZeyEsk3iBeXPDal8acNCBtw/0sW6HoPGIvMZS0gbjQdes22q9+80erUKZrJKxKY4JCtqyddfbp4tmqnzPwgBl1QdM1G4LWv4hww+jRjfO5INQoBtYrNj251c48a41VkNbs6LB3vvOd9uUvf8XQ5/Vaczg8gWYXrSHXuD3yF/NgSjryyGqccEK7AJVAT8N7VGtlARNqzIfJJaCFHCq0SsqaekikyQZi67hahg+q8rAX/EejOgFkJsfFn8XSX3zJFTY5MacOFkpGV1x7jVNRG4HrGmYUsWEIDZkRBELK88Iw8iypp6+5/Ep91g477GBHHXWUJGzdw2+n0ZzyziYMrufeNevr7bPxsTGV2DD6TlsMwFU6LU/IYRG4Qm0fWVUiGiKikJrJE0lTmbZMP+jkgLCylENnsoqaRke3yijy3FnnOC4Go8rokZg/I2DOvlAE0NVjR3/tWCvXvO2U91t9weq24By1e4wCXABq3KJqUnopLrSbIsQ6C5GKxuWEkPu2m79rr7zySpjc58+PMtOb3vpmr90DPtW3lfboN+ZecSzsUV5DM76GnGsfeVeUkzRcjCDiIE4KImopWuL+605qyVITIlc4wB5+IE7FQxMTRU3AziJxJoeLo8F44cN5KpAG+IBY4lHZgf7SojcnYzUV3nZ1e100gF8R/QVM8k00bb/89eM2OVmU/AudFa47lLCvf/2rQoMXL17i0wPZiEHrSXlXl4NTkZjNdYs5E8oWE+OjlmiV7fgTzrPZYkWh3YqVK+3yy9dYPhgO0Go+j+ti80Rks81cCSFLLF+ogyhI18a/c4oBkCJ3mZqsE8QJieGvIHRmVik6F9WNg3teR/C15GFwtkdBrpTh4SEHpjA5ZoXCjOqkd/3gR/bM35730Y8dWVtz7dWqxQauR2CseY0TA7l5yyZdmyRiBC6lbMvIiJ1z9rm6nje/6c32mc99Wt6Wnmc2itrN1CEWdLe0zgyy8kFvhbl5eV5+Z5aQlAMS5hypw6bsbCOMuLxlC0ZVT7uvNYJlvb39CpkRoQMzYM9QNqJ8hJGP4evGTRt1L+wnNbS0kK/13LFWQ9cpTuZzreKTTjpNooJcE597+RWXK0KQqkqomqhvJmA1Cl0hFgklJyWpKIoU040DVfcG+gvPv7Dd8+zD3lp21tlnW61eUkO/UPXgiSXXm9vGw+bCnJddUelRxqMEv6Gse4vpHPfP+/I92HqS8OXgikwgAGTbgOGFEghdWtaNeqF7gzC+IsD09FjyPW6I8gcfIP1gkcC9JQtJDh2AVktkdulM0UDd06XEH2OANSNfZWP193XZ1ol5+973fmKNZlKhK3U8NvPb/+1Ae+97D1Z+Se6LkvzwomF5D8Lazi7E3wBSumTxBdhElhIGoNaw8bF1du21t9vLG0cEbpEL3XHn92V82FyQDWKtDKOkDp3Q3xqNAmsRv+dKBXHiA43mDsqR15Jrce+cVh/9gZcFkeTjIBP4a7f/UggehMBleDRMzZUXiDrY9KxHvUg7Hn20DXvyL0/Zzx76jU8jTCbsyuuu0WhG16JzBQ82iCis1rLR0RF1WLGpyDG5TzbELbd8x1566WV52z332sNJFqE7is+ltkzTARsIYFEU1nCARfsLJSnm6cxMz6jDSnsmIs0IDII0Q/VUzXSb8kXctF5OyQqrcKTXpWR4koThfM+F45taX4BBPCvOQWmR69/rWlj70dExYzby6aef5dzwTEYp2iWXXqIDzz1KDxt1RdRJAoCqSCPhz1CrGDANX1GR/Oyf//yn3XH7nQFdb4gAc9BBB9p73vs+9TsQusOum5mdFEMs18mUQq84COOobxsMxxwnDBtGZXZuWpEb9yiFytDMT5sga4G4ROK+a7/egg/LFHHGR5JtoVAfmRxYd+QwY60MaJsF5IHHflz1m2qaHdaxYLWq53wc/GLVxc548EPDfSqao+bAgsVNUw6EAKkVZDI2OTlmjzz0R5ukKRwVgjINED4I6tRTT7RMh3t9lpB8EkOhnKNMWO9KGfkcxsQROlngUFeemZqwf/zjH3b7nQ/pCWNxb7zlZlk8MYkq9PXStVIVuX94eJErFtJ+RoknoIYxD8UgicqoRnifL0w/L8DN+vXrbeXKVQrTOejRIkdiS7nITFW/Rr54QP+vr1hHJ4SOh4nWwnq1ZPNTkzY9O21rr7pRJTJSiHPOP88Glixus4TwjKqpJh0sRI2QL+RKSQ8Iy7xs41QPDvj8/KyuDSOxZcsWb1ur1cMECBo9OmxuZla5JPeve04mnSSQg7nkHjWi5uSbEYQkdfGKgHsvohzWGw+4aHhYQgaEuqC4eN9tRtIUzipCCaCh6K40uLfQiMrLGUgFZWbWZqenlbsiLnDp5Vdp/TE2O6xcYcccf4wNiIo532a+8XzVNBIQfcpSNIggqgciiYpHviNnKIqyRtdde63WRg30zLhNJ2z1Bed7ZCVpHs9rOzOpNiLeaFRUfyZlIn/m7BD5lCrwsL3pIIUogbrfaO10FUhPZcNgbdoh773may1kPVAz8J7clEZNxB5QNsLkxIQWQECFKGVu+fk3C47FG59gqpmLuUHL48Hye9mgesfGIQfjcJJPefzuvFVChsmpKbXcMT0PdtE/nltnf3jyRc/VJHHqXucbZ52qh04k4DfX8sZ3NHXzOYXGW0e3Wi4LTxWqGGULF+vmYJYKBdsystmuWPtd1+LNZOzk00+xHVfsqFCPh8XCc10+bNlVPQh7hDzmaS30NrG4+QgV3Qv77BuF6qLRhQl2otlRH/ZZw95p5MoQymuCp/p/HVwPkx34wxGLoMEkvZq3zJWYElev2PnnX2a1io/M/MrXj7J93rBv8A0eDbDRoM2Nbh3VJEM+n4MLM8nbEL0VL/KNyad5VuSQk5MTPi1AFEpU9f3QdeUcDebvHCg8Fp+FJhKbkL3BgSeagxQzsmVE/160aFjPTCgw6RiIrAAwNI45wI6qE45u4+9iULy0xF7kOvEu1H5h3oEjMEYGQy55n9k5Ic3c49jYhN1wI8BbS4DboYcdZu/6D8Ta6GiiH9mbHdgLVDk4/D5NsiXPWpFcqzcTSKY3mRIwdd655wZCBAe+Zbvttbt95jOfFV4SU0D2yuT4mEvXUtJr1dWbrJp81gk/XoYEvHTtZv5kHbmvPM00AsYoU7oaqgz5fdce3apX2YQOJiCVUqnA8vDGZRY9AjAiRouQ4P1Er9ltd3v22We1+IRo/NxHS2QUIgA+8KV8L5HQgnR1d8nqR42dWMfDUqthvcoGX1BR++f/86TNFH0qu4crZq993Z526Mc+JiaJM6a8zolECRuPmySkW7J4sZeCFhyBFpCBNW2YpDAvu+JGWyj5Qn3ui5+3fV73Wh20vqDsEPNNrpP37+sbCF1CPk6D+/OSmDPLsKw8rBhKcai2jXJxkoI2YzikGAQYVarnBn3l+Of2xImItup16FYHWRzJ6lTKNj81pbEjay7/ltISNjVTDd79/ve2ZUw5zaw76wi4SJ2WNQEg8Sl+LlPD57Ou7im8UcA9QkXAIsaRkJpwm3vtyQMgEa35v2OpCnCKr8iv5fDDQIu1Sjaz571QZXkGPsRtYKDfe52Z3IixTXroyL1jGOJzlKEALESSNwBhQvxDnoih3mWnne2Vl1+W89i6dcxuv+MH6osmGrhszRrr6e/RffAsqQGr8yxwChRthV5q+MVk8gulgiKABsL1Xd32x8f/YD+6//5w/z6U+yz1L3fI+C9avNjxFgFoqGEWpN6CAin16VU7rLD5BW/KUDtoEBfUtI06Rtlr7ZhKjKaMYI/PupJ0zU+/fVqLmTBC4zro2ofHm9GAXt+I7iHYTKB6tGjRihfDHq/jegmJw+FcXuaUer21p2dAi6y2LRYGLeHAuGEzqCVLdL6WzRfmlQ9pYnqrYX944in7x/OjVmEqedpJHb293XbBxav13rOzMyK/C2TBK1a8yM2GIQTiMEUDgbVmU8c69Y03f8f+/txLlkx32P4HHmAHH/xu6+vvs54e96gYEl7L7/tA5pLrUwk1RioFQgnSn46eR+oaD2J7RJjr4Z7UtRIQ4TYVUt4UL+JhlXtfD4vcUIX+YCHLXprzdjYyE1oXG1YpFG12YtQe/MmD9qcnn1MueOA73m6f+txnFa65IcFD08XE8KtuMb1UzlmAwMBByYikQgcMz5CwlvQoKkZoh6UAACAASURBVC+SEkH/43rk+UM+SwgevRVejnyT/LEdjaj5o+agWda7feTFa1V58mjlWGO8L0aDOinhdyy38QxUMgztlLCgBKRqaDrcX+ezc5iV1kGlRXJWhq0ksPPvf3/OfvzAz6SAggG54OKLFFarYSD0BUtqKDSTKELo6ZH+tkcTC97ZQ5MDnq9ldv31N0qQn3Sq0qzbrnvsbh865FBbvGiRX7uqIR5xcT/cg6JUzUT26M3vAyVRE/9a1Ev0pQuz7dIqpU8MF3ltR2hukOe984pjxJwCmMp15W1gcFjaQXNsiNlZhTaEJdwIFgO9IW3UgBiSvHMBXJwslTZnXQ/K8ycHCbBmsLG4CBZLeWgexYox65E19noobJxicd7ynTnbsHGTPfAQM4MIq50yxvuffd43dD0YCRYAz0EzOGmvqHVwWRcKMjQAV4AvhOdszrkANjz6+B/tvvsfVqQxvHSRnXbqqaK+8X5sBJUGRM9DVBxpWK83O83PhdnxRHikeGij4oFCaU2x94ZorCehspPMPeRct26dyi4R8nedLydH+rQ/jzAUVYjh4oSKgLuAWklxEw8wsXWL/f3pv9kdd93vSoL/8i92/MknesN7kkhnQSUdWE0YEAyOG2gOoYumYzGGBwd0aPk5fFueLZ8PgwyDhSdRKae9ocu2bNkyeXEOH69nraenprVmPGcOJNEFBkM0UhH3TfuBCfQYWW/hc2mdhbl5pV4idiDVO+PyLjxfZv8op+WAhusA12ChlE8H3jKLRW7KYRgfH7UHH3zYnnn2eWu0UgK9zr/oQoGp0VBCc/Qw3eWLMKZCxRnNku+y6ZlJIcystcA45FcvXRP6fVMqWR59/LG2eNlynR2+aPTwqMCxE0Jw1aMR7gspBevhDqDiUxOC6gc1a0lEaY4VHG+X9eV3wZCkvf3zOy9poWTAg+zuZS4M9bmqjY2O2+v33VcbbOmSZWHkxBIdZh5Q9DRelHdVAw5jLJ+4En/C6kb4hYQHC+IFfTFjas5jjTKm8sLE9QxXatRsfnbGCsVZe/yPz9qLL48GnVk6+ZK2/4FvtcMOO0xIHTKX6EvR4UHIw0bFiMzMTNnwokUKUdTMQFRAaJdyZHWusGBnnEljdcv+5fX72Be+8Dnr7emVdQUQEQIMUt2ZVyTA1D02NS10WOfIueWQIsWC9RaIIhX9jIwGQEcElraFwV5bFaQfDmhUN9jmdd3jKpwObYV6n6DOoVxTSKvXhefmpm39Sy/ZFWvWqmtqaOliu+iSS7xnNXhcnDYGLl63No8+wxs3+OyB3h5dGznm1hFyYZPR5sACsoEroBtNWI3UC903ArDKJeWwXsP3ZnCF0t09WnvYSbGOT2TE+5B78j0+FwPGSBNQaLI+RNWef/55HUZVPIJUjdaX0D6R1IHGEHPgqDDgxeLEB7w5DqBaKdmG9evUPLFhEyyxhO3xmtfYV486UjVxDDPPyidUeHSj/aJ2vZR1hjY79gRccgTvuL+nnnzSHv39Y1p9bB4O7+TTT9VQcVoNcXC0xHqjjosvSISePxs1vQfeevkOy329lf54aZCcXcYyGCcL9EvO0sycI+g4ocTd153WciZMTioKkCLwZIRBLKZD1ynp5bJBPY91hDDX0eVNBrS4gSTyPbwNYWtot+vu69Wh4X1HxyfaKhiUYQiZgMyxfj29PbJWqO17aapm83MTesB33/ubdkkEz8WDP/e8sx1NTPiB4XdYJEI1RlosX7bMNm7aJMALhQi+6MFkqgB/0lj99NPP6KDv+/rX+USDLMp83TY3O6frrahTo0fhEfTHWAYiJ+MACGCq1rVhooavuocqVX2PA+8lrj43dIEhFi09axQNnyPOHh6367ihruu58fajM32TRaQREGdkdL2dc/aFyqcGh4bs4osusmTG5yU5m6elzc51xQYB9cuqVu2gGpxh8AeBlJq106VNRWkHz8i6cj/i0Qq0c7I94anWX3IwKRkCn0CfkaFns4k1FFBrDvusWuW8g4fmj5WrVskQ4+mXLl2qw6Mp8Gzmri5J0PL+XpGAI0AImbGZkJ+yRgpLg+wMnHPC6S2b19uN199ko+Mzlkhl7OD3HGyHfvRQa9B2SQlIE/e2TWpk34lKSQoHSYTcWuW9ps3NzOi6rrvmW5JaUqkrmbQTTjzB+iBTwGnPgrJ7js6e4F5UbQpG2IFCJvwBotV0b6Nbt8pB8Jooy6soJCDnRDviXTcaqm+zfomf3HZhi2Qez4GahLOjGCkYpu9Rv2V8paBqs6VLlkpAm79X6VlVztohDwOXVA3QeLS5eW3KVTvvpA8Tb7fpJQJCy9l5FDOcUCA9KknB+phFrCULB3+22Sjb9+96yCamPETnogFaPvXJTyjsmZqdbOfXbChH/5LqDIphFtgWjfcMOKZvk02KMr7LdHpLIA/He3H53S73sl09CsM4sPCvuW5a77zX1GF8BmMBiBFCDQzQ5gVwBed2Wn+Xoh8i2v39MkwAMOqL1ZDqzYoKVNjaLjzmgQlIUwdbrBNvk+l0rnGYsEhIXuf6ynbiCSfrcLEZ1q5lHMm2nmoZHTMBdzFiYB0kM9rtE+5A7oiGqNFiMCmXsN4ukOdi9BxoSmSvrntV9FMOD9dDvsyBJ58FB/EWNG86YJPyPKge8EyEnNar+j4HkfQrln2oZvh11drlJF27DrDLFMWUjIOe0cR5fx4R6FODA9GeiB5NO/HkkzTzN9PRYUcdeaTttNNO1tPX3R4Y7kqOrrAiyaTApKKGzhfrRUhOjXfzpk1215136TPpu013dtipp51m3QFJFkmkUhZar30TniPfJ3Xk2jXcjH+Des95rZ9zgKFiD3leDUCFk4K1GAbOC/Nwud3EA3dcJsojJxpuKDeAu0cWJOorp3KO+gmc0OCshHR1N27a0EZVyXFiWURsF3ltzyPwOIrnO+kzdI1eNTGEw0CeGRHJUpEDX7Mli4Zt84YRm5vdauOTs3bvvT9tP5xyuWp7772nHfaxw6ze9HoX/7FZCMuY4aoQE5YLigK1mnIxQDVm4fJvroNNBljGgWKxObBYOsIn1mNqhnqnayBJlLVWdyudzcmy4528tIO0aFZIdjx05Hnx4OKxly9f7p0mvB8Qf6BJ4pkIaeOsIG0+SeU43zcizK7cEL2ue1yMppfEvM3x0ssusWee/psNDw3bBRdeoNEVPDM3TOT/EPKZ7+O90GwqNjk/5PPTGTSavEykdchkbNPGTWp/5N7F2ir7xDoaBRSoi+hPf+yCDCoblmdPuqJul1Dj5hoAHbkeqJSF+TmRX1DHEPIaJkIQwRA5DQ8NCXhcvwH5UydOyFtlMup5Rs2T0JW1wuMT9vLzKOYAAozXQ9HigQcfsod+9ogM2qXf/KbLBNHvHO5ftfgwHV5chihC13R2mdawUbPpiUn79a9/bU//9W86H6z7hz9+qO3z2n3UZonDmhifCCG+r4sojxIYNI8GUQOhsSaodWjPMsKFXJq6c9DOis8+8ptFxAjMN13T3TevbmGtWCQW2vOJpoYUUfei5zXWkLiQqMHEQYSooIG+hK+0e6E5FVrAfMM0BSpA8BfPMnRBKLw2J4uzkbwe6nImWFAWESs0PTlhhblZK5Xm7bbb7rZKVfibVSo+OOsb3zhFdDwOaxQJw5qh37NkyVJHYTmkUTS7s9PDopBfOs3QD4NvXJ8WoMHeoS2O16vUoc4npEUyolYuFLGq3eoBFlraiSbTVtt9993VZM3G5UHwXhxOQs04yYADDW1TTRvULSs++TxeBwupxoXwwD1UJix1EXGiCnFnw5BoQDmMAtfOPbMx5a3D+BR+l++DTQCm0c5HLZV1Fxm/XcpquTHNuNfAC3JPIKWkHfybe6F5RCWJhBNhAFjEpAp1fg4kkQLrRkjLwfJIzCVvMBpEVj4LykeaqM85iBQqrcFwpJl052QYPoP8j+hN0R1zkZnDCzc6TLHHywoQE6vLa+UxR/aupAFhHOL6Jj2i9CgO0NEb1ON+EFspUHxZ73Jx3sZHJ+y7tzDNsKa1xSmccc5ZTv1U77VfZ+TCtWceg8oXCsr52UfqE9cUBFck4SC7Z3eBAHJ9DjYRC5x+rivyHhwHSVjiobvWtBgx6Vxkkmum0TWtkWhaZ65blpzFcGU/V8b3oUyIwvnsl7gQ0VuACBLqxFY9vPHM9LQsBt6GUDbb6eUUwh82EhcDOIQV5RB70/SCWtnoQnns8T/ZY394UkbEZ+Sm7MijjrDBoX4hdlh5HpZ6cxeg5rkFhjiBtYttW5EYTwjiuV9TVpVwn993BL03jNx0obFYp4RiSU9qXz96TS3lwrvtsbcOHR5WZZX+Pv2dz8SzsSasnTwmn1XzLpdVK1c6zTJwwHmAnuN67qoHRT4emGF8H91o7pPnAT4FRsD6z0xPel4ZIifPxXXc9Z6RfgrggVHEuCl/DZJDft39ogyKg02ZLvT9ToyPO5NIw5l9jIlyZJWTvJbKs2PzQaLh/VkDMaVk/NEYg0SQtgWV6FwelYMbc9Kx0VE5Dg6gpjdQmhTYWdckO3jU3DMeSyIMoP5SHWFmL9ex4OXHUGbhPRj+xvvEBhb2AmBoVJFgrahJO4EIMNJJ/eyL2C+LjpYbcP6vZi88/7L94Pt3qwIDR/6d//7vUgrxBhQOPVx+LyG5fDBytB5NxsgEOi1ALfsUI8nzi62ArHPkLHjakdbBxYjLS4f2V3ETCJVFPVOZxiVDlDMglVEs29DwYhvoHxRQ5cBEXhuG36EkRElk8eJFNiutWQcmWGSsI9aHkEYxOpZNbW8UkskvPPTBU+G1hUiHkYtxRg5Op1YuStFw3boNdv0Nt/iUd7G8Grb33rvbRz7yIb2/K/y5BUces1Aq6SG47AfKBt7xoQNLaBg6PVgMrtfRPY82+LtI5gAUoJa8V2fegZaBfk2B33XX3RQ2Tk3PCQySqBh0R4TGOjoEtmGQeChqN6tV1UWjqXP5vELNZ/72jHKZAw84UPegUDp4WylKkJMuLOi9d9xhB3l6CWnLmHhxHw9EM3zMg2K5iAcvFYlgnOJ98dxceSSmF5R+fKbt1PSEDrBqp8H7gETHLi5ycn4WW+AmJpiRO+RhNyywUKfGQzt1Mi0j6sQJBqF7PzHOAQQboIe1IqfdsGGD6I6sNXk/e2l+jqnvPhGANaDUFBsTiB4wPvGQz8/OKn9nXQX8BPJDYX7WwUPCZnAJOtF6eqwz12VbtgC+dqiZgc/j4PBzR++JLd248FVr1tTNdc7Z51kuS9NMwk77xhmWD2NGNGm+XlW6QN6q2Ukq73hzSCz7EYGgPY3zIv/n/tgPrFVspMfAqhRJpBRok3HvRr584kffu6yl0EXuOKML5hdgTnnu0KlGcw+38AqxgIzndC4mm4nQNr4P1mjRcCjF0PkfSNKx3snDQic5ItSEztyItxB6Us8NYZHYaAAuszMT9thjf7Bnnn4xdNI0RXE85fQTdYB4LxElFD7lrVh2Jg8v5nuIgvHwo1wOOTq1Xg8LfTQGm4tQ0nMl18OKXi+WTJRnZbPW09tnS5cst3Taa71bR0asp5/m7U5xlMmXyWy4Hx18wLLpGUH66vrIeWSAl1g0vEQlBUJRSQBpyIELsRNBM+aRtePhY4Q44MuXLW+XimZmp2XdOS3IikbVB5rGly1dai+++FJIKZhQx3QDrw1ivHRdMzNyy0ReAuXI18TbriospguM73GIQUmdUFO3gaFh27R5cyj7lLUPCGPj3CCfUuDaWy6iwExbryQAYIk1lUqqbs+9EplheOMeoPWPgyDEP5AyOEQYNcJhSRmFEk4k4uAE5DWpPde2TUXwkR5uuB3xzqkzCU8moCkSPJQmecSDSotmBYEnbBedUY3AmOy7776qj8f97Q0S6GA5b53rJudXX3Ag17A/XEklODmGdisF9W4wIpioxhFHjjhD0NMYnAlGIfGTO9fo4HJx3d1O78NS7LXn3vb8Cy/oge6wYpVYSngvXudzQJFc8Q6N+MEsLl/Qvcjv1LIU3o/F4CZk9aQ36zqxWCfek4VAw9fbmpyxFRX7CbXGx7bahvXr7ft3/lAaQlEB4evHHBXC4G7p82DRmE5OO5rCRw3faijnJcSL4SgbSXB+AHxY8CgSzsPn2tuatlGdMqh3gE4K/at5SEoIjbUXEIaIdtWjDv6LFpjPldxL0eVNRbHLddjmzVukErF8xY7aLNpMKEKE+jDX5F7B0Wz+zXpxSLhHDgossfiFCke0ypk0RsjRejYGUYd714ZyWIw1hjmG2Zo+MDCgtIEDTJjHsxDxXjUNJgV4OZDfLWqcqOsBA0Byb3wW6ChGgGtWjZRDgAcNhA48KgPbuA+tSSibOTjjmtwcYkTiXL+Mg+sbXDgAZSd1yczLK0rOt97QgQc3wdBzTzDhRIhI+GxaB5kQ6+/TKBLXE4tSMj6GlahQTkpcdMLcbc0RGB7Wjb0TcQOF0YFJxnPaHvCKZdLI6WfdYq3Pwc1SEJh3iSYdSPjQ0qqecVVNgW7cs5f0MEhCzR+860qhyiwKibv3vjKR28EPFp2DouFJRW9aj83vxP3KS4JiIIuANaSlTAJe0tXJtlvwonypfr/sdVEOKEgvB3ZoyBuL8XYuadKlG2GTzk5PaF7tj3/0sG3ZPBbqmGY777arfeLwwxXaU0cjFOfArVy5wjZsWK9Nz6FsAzZBYDqCZzzVqE9E2KoNWSyqiM5hZD0wHJLHIT+kuVoHOWGLFy1ViyH5Oxt+enZGeTqenPVkU4Im8wBZDyHdDdMDIb9y8GdE2lE77bqL6nkCVBLu1UFcIyuJa8IgRuSe94ujKXffbTd75dVX9bO48dXAX3HJVw4qa07aIo5w1TefRlqG8TNCzK0lMgThN0Z03br1Xr5iHAeT6oLgQQxdKzUIFA44Ue7ivdjYTmllH/kAa/YQeABGZK+99lLoSu1206bNttPOOwmEZG3Gx0Z10GNr5NLFi9spSFdPj6IRIhUiQYnei/bqbYkC7wK6z3uLRgn9NnQPRa9KAz7eGULN7KzvUT+8pAwdGvki2iRRaMajnGiQKOdg/FlDdSjh7cVDQD+cUlVJRhtjvXnzqK1cuTJQOSHpIEAxrOuNnykuROhVdnEAxoQ6YwyHE3W7uGfSCowv16gJgb+8/4YW4QCHgxonb4Rbh7/sOkD9No/anEYzFGzVyh1tdsZnp9CRwYIhrk1xmvchNCMEpMYWSQexw2Nqerpd3iCfYXH4fTY+D165cbeTGTAQgDx4CGiKauFutmzdulftttvucBCnRY9qhx1/8klqII+80wjD8x4Io0dubkQ9IwiBd+MhRBTVhejo/3UpUg1xDjNq2HRxTi6bVSGX6tg+uY3rQL9Xqn/kcINDAmswALxGiGc2o8OD1+JgIYvD/XPoXrvPaxXV8FpFMEGtYnJqQvcVw2hCcA4HXVQ8bCw4+S/q+9G74X0U7klQzdVFuKb43soP83ldM3+PKUZPb5cT+pFuEartSK84y4FPrWpCt0/Ac8wjpDZdcNgn9Yzo2WXTxUPFvbJxd911dxuiHFepSO+K+q16W2HepQEG5wOg6e2RFP4j7ZG1IzReuWKlHAHvzT6VMlGYmAgOgdGMaDH/pv6u2VdxhCXRkLrbnCQSw1KtF+iwaKeek1Ka4nDJmAZhAO4PcIn8Wg6ICEo9x3hoz42JbMi11WJIWhiINxxMqix8eQTgiDZRCgdWbYQouYSxrDHXJvVRjblU0rlQBPXgXWs17JEfMmaDw0bdjgiSjckCLlqyRHmbtGeDcgULNzDg4SgL19MFAr0tN+OwKZfr7DSQSQ1SCiUPLG5nR05yJ5ETDMghS5JMS5+KjQ4QRrsgpG7lK3i+uXm77rrrbXYWhUGsedIOPfzjEvCW6DYHIoxu8PCfMNbHo/BweN+h4WFZbLeqHpoJYg9av5QuhCAX5uW9o6aUPGYYQA1pgXo03hgQig0/NDiszxCPWTNnMj5oOekcWWp47Y3AxMICD6JPv0+3kbScQyfPyJYtHq6LMeRDwvldlRSE+Pq/QUoxMG394qBqyIPm9zTLdnBQFhsSjUJfGSMvufAesSTV1+dT5CIUHRlw7A1KGD5Hx6fIybsDGs3O2dDwkM3NOrWU9+rp7fayYhN5Xu8K4lDw+0QNdOzgtdk7pA2sobqOJNnje5D1YCPLcBRLEmEgyuAZq2MLKSBCaqiFAQvBAPMzyCGUsYh+hhYt0s+5T/SkWb84PsSBwKbjECE9QpdK3lsaXdt0sajju2SS66ppRE44fHymIkzhDN4pxl5irSgDqsOuCX3WAau4jvw75tMKuSW4j8P0hvnwIByFl0H3MTgY5sRDP7i6hfWQNEkYzSE91xQ1NBdmLgdVR8KJHMoSaBgpHNqmESw1Wak0kB/5IKyYL0dPR/4QifiIzmFR2ORYEc89E6Ii8n3AF7yTwnb6GFWg9+6O9es22g033KiDy3Xstuce9qFDPqJDyesxJEIc1e/bLdYLv4vnhfmF5cMo4AWwum4pPWRSGCMFyW41PwvoYWg2k+rVweG9sRGaj3kb90hfaewI0XCpICbg1txRXB7qDkxKn5wUQo4n5GHKC4f6Kd7HqY88yEIbrYWUwOt5ba1GiOraw2xijMhee+8VaIJ0L3W258KqZS6Q3rlu5U9C3D2EjnnqwoJ3VLHhhgcHReoXaJn0/JTckL9v2rxJhwKjBm7B8xobnQhlvLyaNYi4IjhFXVec5Q5+5iAi98hhxejwM0UGAJzq06WcBxMqKfaW5GOQPgpD1+ANq8QVOMbq2qrVbXxivL1vqFZgOGhIUCkmcAqkpIEqxbR3v3H/S5a6QDkHgrlUQoMVBi+0CUYQhiKRBWejkmkcQK7JGa61jcHnekhz+LmrdlAtIAXyPNq7rIhgQZgH5ElVsgyCfP5zb1mNgC5nkjIlLlZ740d3rRWtQ+1wuS7beeedVfoZWjSsXIcL2mGH5QGE8lYpYnh1uaBYqLEPxOqeF7CAeEM+VCFVyXMCHfSG10yxtj5P1DWN8N5sNDYNrB/EswA7IDJQVuGiG1JzNL0nr6c7o1Bgoh+AQtbO+MYZIrqLtSUVDpBP71DR4jFZjsgAiRwAjyCu7rQ838hCtfPdCpVFZEDnCKUHmrYVevqBEmAQh35r4rlHJhIfQENYAu2ICvjDVWjOjJsGEj3eVifBsKAjrNqpwAlv0GdTC6lX3ZgGBxcOJ8Tj/nzQ1oz+zfswo5XrwZsJIBGxH86413H5TIgo5HYoNsS8LZZ9eE3cILxvDKnVgkcXF/cS7hFjEUE/nAI1WIwk1xvzY1InDoL6o1MeNRBOUm9n40oNEo9a8vk/UeKHtcX78W/xAIICKN+X5GqvixJiANmv/eIf0KGVs+npMBKF0SYFat2wAEuaOhDJPSDYqslLnZS+VkaXIL/TbHPlNYw9MLCoHEiONVQSeD93DC6JxLPCeVHFYE3c+Xj/bDrp2loe+XjXlzqFqLA0mzJSNLrwjIXgy3i7cCLVEkWPqFVmaOlzuVmBjkEuKvHLB2+R4A6bhXsBIMITkRuwkVhIwjLfbJ1SAwC5w7tJTKtUbBPzuSlp4LYSYhXFRgNyMg5k9KocRAe1PJ/i4rE6nrT78CbAEfIVvg/ZgfIU3tNDu5r97OGf22//91HrQHIllbArrrxKVpmNKzkSych4aB05tHgnrCpGBoOiujGjKygvhEK3y6Z6mYTP8oVPKa9nLbztzj0714HCh4d4zmwSQ4YGAwmm+b1E7xb7TGMvLNeJ9Wajq1QRuLh4FvIcrsU3LTK3PodJXNhSSd4KY8drXQYXxpnTL32WLlGE58saZyn03NUjMURisqWZBtEVpIjmJEbA+hMBqbc1tEy64FnSmXIqw3h+jXAbeSnXHUdv8nPqvoTD3mTviv+xOYBoTTKooUnC8zwP+1U7DyguOTTeFnIPa+NtkhhJclTPodk33BBRCOg6ObaDe3QU1WS8aN8B5+AzyIcxBtKRAmkuV6T0GLEWFhjPiuHmnoeGFjkmQVQSJivKgIeZPy5BhFekf91VXSI4mWx5muYgYsL7xoOqpXdlIcjrdWM8qWYFB/4An+FVAxp0vOEj7jHuT/nxQ/ddL7E4z0e7xOkdGxu3WsOJ2yIwQE0MdDo+Tq9PJsRo0thCrAxhRo55sj4NnA3FwWEB8b54Bw4zG4mDy8YUZznr8iLcdERteS/4qBw0DozXZZ0YEnPVjRs326233i7k9JjjjrVddtlVjeNC5BAOr1fbmyl2qAA++ThFZ1nxYGP5ieuIvN/22Azau4LeMg8ecA1LiYohm5V71EYMetLx4Ea1CZVUAuvMx3e4mrD3ETPn1g0J60kTOgc41lEVSqK0wcMLYlAYMgwe+RiHjlyIPx008zICmxEPhFHU7FhULTTp3SsHkSnkNUyPZvh81oH1xVizB+L0PDWHMMAKemAq6XOLNMmgU5I2KtWNjyvSYLOxyblXZxOlbMuWrerUIvrBA0stRU0DaJI5zZAv1oTDzwaPVY5i2BdqGYRFFsp9tMPhXFTTDFPsYmTDtXmNtyED5IJ0/t5DADtoVhtig56i8bkcGtZIrZkBp2GfsK54eYXqQfVF7LpZF4Gjvc6li51Drbp0ULFs1pqqKAiwQygiGHAZIZyPKMNet5ZHDdROno83y4Qh5DRjhDWKfdPKoX96zzWt6HUAZXbccUcb2Tqi0JTNIIQxlWz3XjLyA2CGDqKF4pysOUAPelIuPpYSUBU5n4wSwUqSH/T2+CK0lQdCH6iG+DYa2qSEyVE931vtAHdQcHBBMy92t5x9AxId6m5sLLV0wX2t1qT4wKaK6vn8HpswCrv7FDQPPWMdWy1dMLNc9E/DpllUQhgOY+Qts/h4bTa99KBD0ZwSmvjWGtTkuk78G29AOAuiypsARsVGc1BJDAgglk809IZuNj2bAiPjh5v8qEMgDcCLG9WGjElku4iGlAAABCRJREFUHLkAuAOCfPEMYo/00CDtmgsqW6E7heFRvbzF5s+rrEGP7Z577hk4z82gPwUN1u9TG0rDnV1vC8EC38hzWicOBJES3lLtckQIGRc6wGPCGHIUviBjHIEZ1p/35plyT55z+8wmx1JI0SDZZJ1LHTqzWF/RalvNNjEEZxD5zUSJpD7kwp6COKkldhdFAAjsAqOAB6fCwXrwGsqjXBdeE2A1aoJTHpXWVRgMx30IeAq4DYeUZxpZXdS1Fa1pjlVZxoQoTPsj7EsYdZLMRaww39XGROJ0DHCMOOlCketvH/quDi5vitQpC7t1ZKs2VqzR0sdIvsfDQrGdiyT/heaIM1CPJ8RtwBRCX+b3dNMSZ2pWANRyDm5SHov3jaJx5DtsClfLiKJrPkSMDaiQubAgYbeIytH4oOFJ2w2X8gHEAC/T4X2cYeJe3bVs1RQQCtqE+NLUCg8yymCqplz0MDpuEq6L0hSHlUNMjiTygggGSK24hCgbS/U2Sb26zjSGI67X0mXL9H1J0kr42r0NuIAMAZpcMnquWQyAETm/fJ+p6q5i6WU0hY9hDWJrIjZE94JiBV40IK4uyObPis/HoLjXHNc6iElWWNDrBdIlgkZX8BARVCRS4Nrd27nqSYyEmNTI+4JLKH+UtIxPvZDHWzTsQGMwyBHg4/f5OWGyWFuBcBCVDsWTDmJ/3D+godD08F4YONoo8fQu8ufKGbyXUsCQa1ZDjdm7pHwNJRUj3r3rb0e+tOeSTq4gxdH0yNCdBHYgrAE1yaCGKU4yfduhm4jzQmUF58L94d2JcjylcoFAOZogX4tmG/tAEj9MhdBEDAeAo5H2PdzlQnaP/eKOFofHSxcuw8ILyJvk7eBapn1GEMVyFCAJpTX/pVbWJlfTr3RnAy+YDRAI77CMsHxCfFM+uJeNF9viVOLo7fG2qqSDEIAFHAoWVaADjQ1dPdoIKpHUnZIWPRNWnwdFQo/VxJjMzdH0H8XcHBRjcxNe6nfDOA8PXbzkozpynkZ6R1Mlxr7dRAMvo3iow/vBPeazI9UzDiMTN3e7vC0CRmIJBfqjxAoS8KN9GBjvx4Fg8xEGUq/F8OEJvdifkPdQTTWQBoRkS8PJSxO8P/VRwMRRGq41+DuntVdOzGiZMJOHDeKAYU20RaIdZzT55uKwSQo1oL9+nWnV2+O+KFeK8q5qpaTPFK1r5u+EEFe17c5uB4OIiOgiChK6sfwTh8Lx3jxD1/XyWbWUsYg08Oisgat3NCSBxHvHvJjXy6BovCtRlbf04RBE+glD0/g7835cAgc8Jsw9qjnlF1AxVkD4GSArnpUDRB0XY6TSHNTgJFxjIifmCnmDCsqP8fBHYJFnuXLFCj+ImYwOL85DVMjQiKN6MEO0Z+eUQjr0FWq3lZKrcbAuoRWQn/1fbh9VCp+xIjgAAAAASUVORK5CYII="/>
+        <xdr:cNvPr id="1033" name="AutoShape 9" descr="data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAO4AAACzCAYAAACO/iALAAAgAElEQVR4Xrx9B7hdZbH2u8ru/fRz0kkhjRBKaNKkKCjGC4JSBEVERLkowgURFDF0RQREpLeLqBBCk4RAekhIAukV0nN62b2t/j8z31rn7ES8/733+Z9/k8Np++y91re+mXnnnXdmSXNef8Lp7e5Fe9GE4QAOgIDfDwUOZEkGJCDoC6JarcI0TehWFY7j8MeUFgVnTWmE6VhQIYOebFkmbKsKwzDQ0NDAz7MsC/Tw/u6fvpZkSJLEz4Gj0v9g2zYcW4IMFTfe+Av4/VFEY1E0NdbhlJOOQ1fBxt7eEtq7OpHJZVCsaNDLVew90IlUfT1s00IoHIJuWDhQigDBekh+P2RVhRrwIxQOIxAI8HN8PgWKokDm07XhUxVIsiQ+w8GktjiuOi6C+qZ6xEbNgG6GseCD+Vi0aBG2t2eBUBKOraOqaTB1Gy8+di9kW8M11/0cPUUdtiNhZEzG9791DqyqiY1bt+Hj9Tthpy5AJpNGqi6BUqkMNaDDNC1IjgRHTmHbrl3QjT4E5ACi4QiGN4RRV59EPBFCa3Mr0uk0FFnB4pX7kSlbKJT3IKBYsPQOSHYJFcNAUFExcdp3MdDfiaOmTESxlMX0KWPhOEVEohYCko1oMoU33liBbNGHxi9+CTvrfbhg2hh8eKCI7v4sUqYExTIxkOuB0r8XqR1zsbXhHBx53NGYEMlj1iWnwDJN7Nu/B3975wN0ZDVojg+5ni7cdPU3UMz04Y677sT4YSMgWRZUWmjLgGQDsB1ICqCoKmRZAiwH9B/9oz1A14WvigLouoP2TAH5ShmmBfzp7p/g5OOnoVAoIBwK0VblPSY59Fwd5XIZjmTRbuKtJdF7ObTDh/ai7dA+Ez/zfk6f6eeSIiMcDvP7K5IC09Yw85qHUDT8fJ0cxwb9pzgWTEnBV49twN0/vxbxYZMB00CxWISq0N7y8fnRsRm6zucFiXaWeNDep9/9V49B+wAgyzKkt2Y/6WQyOWzp7Icl+wcNl1ZOoSdIEhTYkBUZlUqFl4CMk96IDDlabsdV5x4JRRGLrCgqLFODrmmQZBmpuno+SV4MOuBDFoh/DmnQcB1bGXqeA6z8cAU2bdiK5uZGdij19Sm+MJFkE/Z2Z7Bu01Y0NA3Hph17kC5U0DOQxojhI2HoVWiaDsu2sb8UhRRuhhwIwOdX4GeDDUP1+9h4fT4VqipDVRU4tskGK7MhO1AkCRObo/j+iTGkGlIIDTsaVc2PVatWYv7772NvXxGGGoVtGqgaOizdxnOPzEK6vwO/f/Ql7OrNYlgqjrOPGIZhbY3IZ4tI5/uxZ38Z2/om8xrGolFAlmCaVciSn51OxVSwcfsm6KXdCPr8GD/2KMiOAUmy+QOOBU3TeHNqcgTxpsNgWXnA1mDpWSRiQYwd1YrO9n3Il1vQ3t2JunAMra1taEj6AElzHYSDukQMjlXFTgf4bOJR8KlBfPmweuzsyaKnZKLvQDeGNw9HKGhDzqWRmXMPIufciExJw5cOT+LSGS1oSiaxp6MTj771MYJ2FkeGu1Ep5dE6Zhq6s2U8/sRTmDxmNMjiFIlOlyxTGJktkbMkw5XF9w6d39Cm5o2tSKjqNg4M5FA2DBiGg4WzH0V9IohSqYRQMDj4N2SIWqUCTdc/13A9I6H9WPtetYZLzkPx0f7ws+E65BYkBV/+3v0oa2T4Yi+zgbNhO/jzHRfijDPOBoJxGOUKBy+Z7Ef187nRg+zCJudSY7i1BsuOxwtiroNhh0bH4P6Ovpfefv1JJ58v4uOd7TDVAL+GLCu8ib03U9w/oMhpOxYdNUzLgmNr+NrkJIZFyogn42KtHREt6bmGaUJRfUgkkgd5udoFOtRwLZN9ED/f0DTMfvVVpJKNqEslEYtFodBx0YlJDjp7s9j2WSfijS3YsrMdhiWhUKqiohniojkO9GoVXVoEmq8eaigGf9CNsn4/G7DP73MdDtiAySh85IBUivw2VFnCqKSKH59aj1R9EuERx6JcVbFyxYf44IMF2NOf5WhuGQaqugbTsDHr5h9iTHMdHnr8FazcugvHjW9GW1TCKaedgo49e0ExoD9Xxd8WWFBVen8/VCXIjpIcBjmPiiFhX2cnejvXwjIKOGnGOZBs2gAWorEwTKMCmyKF4+CzzhyUSCtkjkwyRxafIotNSf98QN+BTWhJtMA2FYQiQQQDYcDRYBsSHLsMnz+AhrNPRldrAoVCGjNGDUMoGsauzl70lGRs+7QXMnQ0+YH4wt8j9MUfoGJJuPCYkbjy9DGQLBu7u7K4YUEPDi9uw1H6CoT9QG9vHn2ZAhas2o6Ro8bCJ8lQJQmGbcCxLMgOIKl05GDjJSPwHLzY3IT8FECVkC9q6C1VUKjo7NzWLnwRsDTouuH+rRtJbRvlUpn34OdFXEZ+9J/tHGS4nhF6hhSMhNiI6MOEhEy6iAtveAqGwZtUoEmpAtkOwIcy5j9/PUYefipk1YdiNjcYSQOBkIisAO/LweD1OSGWtnZt8KX3ONRw+ZjemvO0o5eKWLvzADKmD7Lih2QZcNjKIUI9LSihGItgnA4TCvyOhiObwzh5HCAbOi9sNJ6ETl7MMGFZNgxDh2QbUANRROMJOA4ZuwJIBrmHocgqy3ywtkUeTHhdOuAP3p2PSCSCRDKBcCQElY2JsQW/1qKFq2H7gkikUti4uw+VchWG7aBUqqJa1WHLEsqVKhw1ii6jHlI4igBB5HAIql+F3+eDSh8EiSWJoy5DZFlGKKjycRBSaw368NMzkkg2tiA+9hhUKj4sW74c8+fPx/6BAuxgHJZmo6iVYRs6rr7sApxwxOFYsHgNnn11EZriCqaODHO0PebICbBMA7v3d2PJOh0FNECFClMvwbIcyKqCgBJCsVpEpH4kdu1YhkppP5pSDYjF63DFhV9Gb18/PtvdiXK5gmAohO4BBUZwNPyqCsumjUZe20E0GkCpWOHXHejajrp4HVQEoUoyTNPgcwUIIZl8/kWninG3Xo3S/t2YOmk8DEXCZ305pNM6KrqCge5u+GIJNMx9APqkmdAiPtw+82hMa9QwqmUEdnXn8KNXNiNo5zHSOoDj5U0YGMhjIJfHkpWfYvSEKQio4Iir6yZff1Wha2ox5GenLLsGYVJEk1yoTNtFQrZcRW+2DMPUeS+u+eA52CahP7DToy/IGC3bQqVc4c8SuUk3Onohmd6XIPOhhusZI6dpcBBLJIZMyzbx4uyleOqN1bAc4VzYJmxyNgZGNIbxyu8vwvBJZwOOD6V8cdBYfX6K2oBj2xzMhgzXTQ9duHxoQKu1axGFh+C09I83nnEqpTJ2dfVhX7oMS/LxG9hsHAJPB/w+vrDk4WWJFkNGWyqMeuMA0rksdn66E0FJx29uvgQWG54wStMyYelVmI6Ozv1VTJwymhfRkil3FHBI5CQyDIMWmAxXZMtbt25BYSCD+vp6hCh/USWOtF6ebNkm/v73f6Bp+CjEonFs2NODTDqPctWA6g+gVNLhyDIqlOtUHKT9bZDDcTbcSCwK2afA7yeHJENRZAHTZN4f8PtUBH0y5/h0nC0RP244I4mG5mGIjjkKhhnCwoWL8N5789CZrcAKxmEbQKlcZHh03lkn47KZZ2PvgTRu+vXT6Ow4gNOPGQ6fz0HE7+CwEcOQTmexaUcPDuTGoqrpkNUgZN7EMmQfIQoTajCJYv9OdOzbgFhYR2NzE1qTEVxw/plYt+UA1n2yw82f4tjZVYaqhGHLIYEiZAWOJMPHMM2Hgd7dGBjYiqAPCPqTcBxy7WLj0LUNBANwNBNj/u1ctE6fhnFjD0PBtNGXTqO6rwOObaA9b0DzBeG89zSGn34xtvRm8eSPv4rprT7eFzs687j6r3uR8pvQynlM8OUxrOt9+FUFz85ejCOmTEDYrwjD1UwOQbQfac1p/RlJ0abgvUZG7RPBw6fCtG30pHNIlzQOCC1N9fjHK79DtaLB5/MJjOZyL/S3lNZxoIEFmwy4ZuMLwxWG5BmLB5+9/UVPD0Wjg7CVHOH1v3oaa3emYdrE8QjHQq9jyRK+f95R+PGVZyI54ijYugWtooljd1MA+to0DE7dPCjM8Nt9/N/y3H823DnPOJWyhmyxiNU79sEORGFYFixb5Ld0IsGg8Bj0vSzRgquQLLGABOvWbViHancGC5+5FgHFgcMeX/xtuWzh+p/9Du1dFVx2yRdxxcVnwaILpci8sLyIJkVb4U1sKCBHsmnTJs6bgsEgX1QLdBHEg55pWQbefON9JJtaEAiGsPVABu37OxGNJeFICvoHcgypOrr74PMFYDWMh5JoRDAkDJciLm1wzuE5n5XYcBWZ8hUJAT9BOkIHNlKqg1vOaURTywhExhwFywxj6bKlePfdd9FdqMLwxwEDKJbz0EwT08aNxi+u+y40M4CvXPgLZPN5HD0hiZZWP+pSKUhaGU31dVj38VrsTsexZdNmtI1s4Yt64EAHHQRikRjidcPR2DgRDQkL06fGMG5MC1paGtHc3IC/vTofjhlCT08X1m/egZIdQH/GRDCsMtqhTeVXJRBMI5YiHE2hr7sLo0c1YOP6tUzYsHGoAeYi/H4fZNmGKsVx5oP3IkBOLRhAbKAHxw68i5FNCV53XcvjP19ZiONPmoGGuhhOPOdCdGUqGDlsLLLpbmzZ1YXOTAk7uotoVVU0GxvwwdJ1eG/pGkyfNgXRoI8Nlxy1iFoUBhzeD2KPkVEIo5JlkfcyWaXI6BzIoj9fheRYOOWkGXj0rh+jWCrD7w+IvUEGBQeWaaFULonXc0R6d6jhEkT3jJQ+e8fiwXQ6nkAoJN6fSCjbxDeu/QP6SiK/pSAmILcKWSrh+TuvwCmnngwn2gSjXIKpCV6Hoq2XchInQScnzon28cGG6x1DbaStNeyDI+6cFxx6wXw+j1XbPkUBIZiuN6YX9zwhQUpeG9vkjc4naBv81rlcDls3rsG5R4zAb/59JkcpQ5ax89MO3HjLg6jqfui2jnAwgCsuOR0Xff1USGoYNhm4ZUM3CbbQK5Gx+HDf3ffAMmUR9RQFyUQCDY11aGltRENDHSCVGWqt3/AJLKsevkAIn3VkUawa0C0H+zu6caBzAGogiGgsgT3daQSaDkcw1oBgLMS5G0UYiqzkrdldsPHK7HRoC8mSLTavLCNoWbhjZhPaWtsQHX0MNDOMNWvWYM7rc9CercIORkDeqGIUoVdNtDbU475brmMS77SZ98ExMrju+2fh+GmT8Lc334Bsy5wv+n0h7O1K4d0P/go4Oh8T5dm6XmGSLxCIYerkmYDUjWggjRt/+h0E/UFOXwgmd3QeYPZ007Z+PDdnCzLp/TD1XjiWAZvRggk4ClQ5iFPP/A5WLF+EaUcchfXrP4Bl98Mh1FZDhKi06UMxfP+Rp2GnGnlNRvRvw5HlZYgEAwhHVISCIa4weGzvmKMvRFHycVWh78AO9H22ktezq6sH7fv70JctYf2eHDZs3I6Jk8chFgyCAAXBWK5a8FoLR885JuVvFCdti9MYj4El8NrZn0WuojH0v/m67+HbF5yOYqnAzp1gr8cq67qGarUi0JxrIl5kpc3PP6/Jb2ujrWcojDTDIjclY9MNA1/9wf2oaH7QVmXiSZahUOrns7Ds2e+jZdJpUKQQCoUBSA45UMtlpcXL0LWqfdQa7ucZa63RikA4hBCkd9940aGDIGZu+9792J2uIhiNI18sD7JYnD9wDkjQcsg7yQx3KQoDH320HAFNx7Lnr4NlG1i6aCneeH0V8mUdVd1kOFhiRs3Ed751Fi666GsMMYjrEnmKgObLl67EiiUfApbId8jzOZaNUIDIJAXRqA/1jQVEo5R/qEjnYgj6QujOGXh35Qbsbe9DIhLD2LFjEI4nsGnbLhzIO1CSwxCIxBCOBBGJEUnlRzDgd8+JclmBMCjvo+iryjaTPcQkRmQHd3ytwTXcY1Gq+PDJ2rWYM+d1dOU0WMEoHEtCSS/BMYCgLOHxe29lVHD2hQ8iFAihpa6Ec04ehzETJuAvr7yJdRu2wLJUnHHmJZj9+n/CsEqCA6B8T6GNHMDxx50GvZKCjh7kM/tw0w8vwbhxTcTxIxJOoFQsorOrHZt3FfHsnA5kB3bBrB6AY2XhEPPMgddBou4whCPHIp85gKOmTcWqVe/BsnshgQi8Wq9v4oSTvoThF14Ju60VMSqNZbM4r/wGI61EIopwKMjGRAZsWjZGH3UBuopVRPwhdO3ezIbbN9CPnp4+VMsWduzpRE5twOqVqzBlymTEwkE4xH0QQeVufoLSTKR5ZRoi3QjJ1+xmw7LRly8hUypRpQXP/PFOHDd1NEdWMlwRcYVD0DQqRwpy8vMMl1/ZEsTUoaUgj7kleO4nppqDlYWiqeC8q38LnegZm/JziqiCT2gIGnjz6evQNvF0SE4A+VwfVMnPTt/jZWzLYkL3f2O4IuqLGO2t0aDhUk6QzuexcnsHlGCEa4CcIzA8pg1NueAQeUAHRAYlfCYwMNCPLRu34sGffAUL5y3Fkg9XYFxTBD/4xnFQ/SYK2SoyuRIMUwGR180jx+O4U06FYzkwyP4p4beAmd+6FhWNDlCCTBfCshGNRhAKKQiHA8hmswxnJRAEUeD4FZx53CQcNnY8Hn7+TRxx9LEYPXo0ksk6xJIprPxkC95atBZWKI5gJIxwJIJQJIJwNDxouGSoDJU54eJ/8PuEU5HIcCUHv7mgCU2NTYiPPQ7lagCrV63C2++8jfZ0BXYoCttwUHEMmBUTsmXixT/ciXKphPMufwTZHHEGQJiIp7AFxwxCkoKgYF8fj2Lfnq0wtDwzxQ50Jl+IufzmhZdh4/pOpMv7EAr5UBeuw+XfPBqpxggTTMSyU2R55fXVeH89UEjvAcwydG0vR3AyWhkKxk8+DwN5BY6RxfRJh2P5h+8CKMD2nIVrNFSrnDrpTGRDEQw/YwaUxpGYFtfxZX0hfD4LwUAIkbB/kBfQdQvjZnwLOUuGrRnYtGoxunYsh2YYyGULyGbK2LanH+VwK3Zu24wxY0YgFgxAdmwYZAFknLbNXEPtw2aoLwgpLxoaFtBfKCNdKDCBOeeV32FMYx0q1QqCQQ8qi/JMuUxEnyhZ/k8MVxgpQXSZ0yjVI5UcG3MXr8Ksp5eCDNCrnBA/Qsjm3uvPw8wvTUW8ZSpMXYamFSDZxKGI8io9n2yJUqH/qeF6rPY/Ge4/3vxPhyhqgsvFQgGfbN6BPtvHxIa3aH7Fz19zHkJ5oELlIsG6eqUf2ZGxZuVHMHUDl55zLK6//EuM9Z1KN6qVKtKZNDID/TCrZfhVGUEiqIJRjD3meE726QA7duzGe6+/jkJRh6P4YYrsBrFoDMlEGLG6FJcT6PndPR0wDBnwJ5Cqi0GzVVSUKKKJBLPb4Vic2dLO3jR+9/SbgD8GNUL5bQzhWAThcMhllVXOuchz0jlRfsvVJoYmJp9zQJVw/8wWNDQ0InbYsdCrYaxavQJz352HfdkcDH8CtmGjajswqzpM28LLv/8115Kv+dmz2LSryMgkEkkg6Bfwj6KN6iM0YbIoISL72UkRdFdhcU5HHrp3YACSkub6X110AlQqwTJBSLyAhWRdmNnskjQM7fu3wC8XUCz0wrAKgK2zcGD4hLNRzNporIsjEVexaeMKhEMqKtVuEKwUD4KpKUyfei62bfsQM0b146YbLkYIKnxKnllbZuOJA3DJvELFwLgTr0C2VOVIt/wfrzGZVs7mkS1W0NWZRY8RQFaz0NXVh/EjmxFWVdiwYGhVvrYE+wXxKQzGE+uw3brf0/OqDtCbLqJUIi2BhGX/eAqRoALbMvm6kQPgNbFtlIqFQeKJN6kLj5l7oW9Z3OOWgtiwDgaq9BpUzQAhH0eBQSjxlqexp6sA2ySRzJABUgBe/vSPMGriZCjRNujEJrvkFeXe9CAcRdeb7clNTQQpO0QO1gCfwYMZKgV5PyI7ETm39ObsFxyCFSRWoGL+nvZubOvsgy2LNyXoKFFdlxhPiS4veUg/wxOCuLTZaAMR2bBl4yZolSoOqwvhtSdvhc8JsKF7LBoLZajUxAdNsMHi8o1eLsImn0BMo15BVTNQqlSYVKGLwlAl24mBgQHEQn7s7yshFG+CpgbQnzagBMjRCOaRVCrJVB0Un8rOiC7nDb9+FAgm4YvEEXYNl45fCC9UdiSKsF4mSjzhCUt7HKrrAg98vQ0tra2IjTkWphHC0qULMX/+BziQLUL3JWCbNsqmBVMTkeT5+38JvZLFc68sxe+feBeRSJyFDcKLEyynPFeFY5oIKn6komHOa5nIcCReg3JFY9hnoxO6pqOx8XD4fZQH+/nYy2XaNhZylSL8yeEY2SzhxceuRkXTUSxXUK7o+GxnN+56aCkG0n2ApaM+kYJjlZmIAqqQ5Cp8ATp1A4rUBFluxuYt7+DbX6jD5ecfjkgsCVkRiEt4NPcYAZR1C2OPvwIV00KxVMLcv7+AysBeFHI5FEoauruzqATq0ZMrsUOvT0QQpCgrO7BIrOJCR495ZUEEGZXjCHRHXArVYh0gW60inaf10LnKsXzuU7BM4gmEIkkwWsII8/ksfy/qwHSeLpHkGS7tWfd9DjZZfia/XiQcgUOGa0msirrkhkexr6cAIgYIGXqQmljy95+5EiMmnQpHjaCSyUNxlYB0DuyU4HD9VhyPeLBRDuLVQYL/0MNhJOgFULZHlx2X5rz6rENJM21yqn3mixUsWbcZlhzgheMnkkzQ3VSkcmEP5zgI+Ag2CW9JBrLr08/Q19OLsKNh5euPspqEuTPXy8jMwokDIWN0qKxNTsiWUJUcKJTbUCQmL6dbkH0+UViXJQSkAG6+6UZU8n24+LqfoOyQ2siBZDgwbR2VquYSHvQ3VI8G18wIkl13+28hh+rhT9QzxR8Mhxl+E5PKG4QgJW1OVomJTcPHLAlYpCoSfvf1VrS0CXLKskJYsngB3ps/HwcyZZihOi4BlHQTJknaHAe/vvZyjGprwPtLV2Pb7j5YpgPTcGCYFtIDWVTKOspGGZV8EX1d/ahLtXA9WcBHKtTTcx3ouoJYjMwzj0J+AKbhhyrH4Q/4och+2I4BWY1AbRiLpoiMvz75HT7eQECFLSnY9lka37thDnp79wOWiZCa4DTAz+UuujwCTdF7F/ImLFTRn/kYt1w0Aqee0IAEIRN/lEk7TmBk4jkEE7+/ewDTz7oWhaoBzaji5T/9AXapm6FqNl9BoWgiMmoSPtm8BZFgCFFFRpA2L103xxICCTcKUTpWy6p6m5UdmSQhU65iIEdSR4ed96I3/4iqriMYoDx0yHDpNSnieqUhQlK8prT3aiIuMc+f9/AMNxqNCqEk1YR1BZfd+Ai6shoss8yyXK+Oe1hLEK88eDlaJ30Ztiyjmi1wGsOkrquWMmxxrrXB/X9iuJ6he8fL8Pmtvz7mFHUHFc1EqVLm+tf6rbvQm69A9gVJzsIqHM5xVSFpZBgj0cUX5RQhxwJKxRK2bNkCx6jg2m+cjqu/PZNPwjPcIY9BjsuVmx2iYZZJ10nqIVa2uAbEb+hg9it/weN/fh533XcHjNgw2FSy4ryBlFyibkwPikZ0POSMtGoVT7/4KjbsLiLUkEQ0HkcoHkUoFB6MuMIjk6xTASlj6WvWzhJ5IQE+MtyZrWhqbER8wrHQ9QhWLF+MeXPfxd68ATuQYqOoUv1OE6TI+eecgW+ccQIKpSzLIelBx0JsOCl9mEF164tk6PRG9Ds6hXSuhFKxikymhP4BjevDp37xSPiUMhzbh3S6jIFsDh3tnejv70P7gQFkzDZEI3EMawghlYrA55PR2tKCiqni/cW96O7fCccwkAin4AuG4VcDzHIqfhlUDqRlLJd02DCRL27AQz8cj+mHUXpBjs67znSph67JrgM5TD/vGlimjWK+hNee+T0qxQFUqhbGTjsOXekqetJpLFm0GI119fCTcyZqjYVvQ/VMj3xhYyAipiYaUpAgdplUcgPFCkzHxsjmFN565bfQqkRaimqHZ+gkIS2XCoKpGvy5iHOsU2YbJ2XfwfmmZxQE+Wn/hUOkUVZgwkBH1wB+ePdsRnwCFVD1wWTE9Kurzsa3LzkewcYj4FRMvsYsgXRhMr2up0/mczvIWwwRg14Er/31obXbg3732aLHnb29Rezut3njFasV7GvvwNbdnZB8IRH1fKqraiHjpbrVkKqKYJuAKiKSbt68GVqpiIRcxtI5f+Z8YjDiuh5ILKJQYnkP78AlRXj0SqWKUHCoAE7L/OnmDdj+2R441QxajjyDYTY7VFcaR8ZApI4HgzivIK1y1wDuefSvCDc0ItXUiGA0zLU/IXEUOS0bK0dfCSrLBQnKCKilysAD5zWjrbUZ0XFHo1oNY/VHy/DevHnYla5CitTD0nQm2ei4CU20pSK49Yff4U0fDoawa+dOTJgwwd1gYv2IlffIBzoILoPQktimEMEwkqE6pMzFe8OgRg+dy0UiehuiZpnpQX9/Gc+9uQ29OQOmYXGEN9xIWjUIHSXQ17MTjlNAkIxXjUCrUp5HJQoiIKmgI0NS/SiV9uDF20/D+NFJ2E4RPjkoUiZeZ8GU0rGtWLMbX/nBr/jY8tk83n71JYwdfxiUUAP2dvShK92DXN8AlixchGQiCR81oxCooLV2RRdebuvVT739MFjjddFPX7aM/nyJhUGXnv8V3HzdRdCqGsKhgGhIcAk24lM0rcycRa3hivRMyA5rm14OsiMBqhmxEdcgCmoGlq3Zitsee4+5Gk4XmVC2+PfL/3Ijho2bBCXQBD2X5+OgaxIIR8RLu6UkjiT/pE8eMtxDj8OzGc5na0p23jlJBz563jF1DX35Cj7emUah6iCdyWL+ivUccYPRCBM0JLimjU1Cf853yB+RMscnch6XHUdXVxf6OjqhOCbef+5OJBNDxudBB2G4Q5GYWEQG0czqEsRwFVI1EZeEGUYpi83bd2Dz8vcx6ezLYHXUJFMAACAASURBVPBJUQRwSTJaJK/7ggorlMsYJgbyBfzi3mcRbx2OaF2Kz4maC7zcypPZ0XmyGGDw/BQu0RCsu/9rTRg9ciRCY46EpoU54r4/fz72EHwKJOAYJkxHZpaXan7JgIQ/zroVlmPAJ5G4YUhg4F0kigCs2GLn4fHzDovumRxwyJS5rUUoXQm9sEMhdyK6ZugfEWoWlW4klXQg/HeGabNm2zaqLM4nKSqRYNVSFoZEsLiC9EAOezu6kM0UOOqWKsQtqKhWC/jWKXG8P+99zDh6HGZMG80IhYT8JjU60DEDWPnxAZx79W0swunuzaC/vweFqo5cOodcMY2O9g6EQ1H85aWX0NjQCNU2IdN6knF45Tc6drd6QYdeK4Qg02NVFEHlos51XEcGXnriARw5vomjG9dwXcUUfSaexrJ0l032IrFbu/1vGq7fJ8qEkC2YtoSb73oKyzb3uVSpyzzDZqJxyTM/RPO00yHbPpQyGVfCiaGI6xmue9H/VcT9rwyXt8AhjQdS18fPObRYtOGrpo+VL5v3prFu2y7s39cH+AMIx2MsESTjJT0sRWF6iIglDI2pcdvi1/ls+6dQZRU/vexMXPJ1OinKlwnGDhmrp0cm+BFPJoSHYwvyNjA1wAgWTexFyqJlzJ07B5n2Tkw45Rw4VhimQmSGDcu9eBRlCS6JPFo0O1DB/me/fBRGOIamEcMQikcQcoUMg4ZDqQBLHsWmFBFRgiXb3NJ298xWjB09AuEx01GtBLB6xVLMmzcXOzMGrHAKEhFTJCYheK5pXPp56r5bQfXH715/G0cs4glCQT87wNbWZoxoSDDhNXrkKIwZ2YqoP8A1cDIM3ZLhc0j2Jwg6Ph9Sj7kX0HbIcAf7MYauO62fJNaktsBPZQvO+zjrcL04i23JH4jfkbabriWhDSLk6BpRC55qmUyO5fJZVKv9qGplDPQPoFx2cNzZX2NisrtvAPs7u1Es6yiVirh71p24+qrvQfUF8ecn/oTmVAphejOviUWRmARkVEHOyJXUkiKJzlE0CIhcmn6fq5jozeYhOwoWvfkEEhH6W2ouoDyf64lMDlCLH8Nk9yJSXsuojzMqcf619dta4sczEHLqvC9ISGRZOOfKXyNTFRGU9xqhMBs48eiRePRX30DzmJPZWZZzOf47Nno3paS9eBCa+Dz6mI/YhfPu9R00VBdJ/JPh9qx9zuFNQR+mwdEiW5Tw8ltLMHflTij+CKYeMRWf7t7JjCiRIvFEwu388fpYRZMAlQmohW/7th1wDBtNEQPzXvoDQyPR4TDkOTyIS9G2kM8jmUzyoVMOzZSW46CQLyIeF0JvWi5SAX3w/tuIROphGjpCreNgugw7HT/lJ/T+XnGcFo3E9ER0zfr9k+gqSmgaORzxVJKZcc9ZeGQURVeVWC3PcCUZlmTB7zi4a2YLRo9oRZSaDMoBrFy2CMuWLsG2vhLscB1V/hmmizyWmiscPP+72/nrS39yp7thCaEIpRZvGHdN6Ou2hA8NkoWpk4dh1cZdWLlhL8PJUDiCYCiISCSKRDSIQCCIRDyBpsYYhg1r4xbG1sYGpJJ13FssSSoz5HTuEtUy3dqhR76xQTuUR4quE2om4fXmHlEPFdB5O1AcarhQBGHIcJqgtIyqVmFij6A2VBO2IWNfVxe6+tP4aNUneO312bANDTffdBP6+3vx1OOPY1hTI/ykTnG9DfEGQn0lHlTjpPIdOW4my0g1xShMkIx9uQryFdGK+MmilyGZFShqDVJhMYWNfD7nGq0LlV3iiq6HMLyDO4J4b7lr5BkHrTedK4lhDEvGGd+dhXKV0Jd4DVuiNhsVd/zwbFx20ZkIN4yFSalShbgCWxBmruGSymwI9oqU8vOgb609H8QJHWLQ3jlI3Wufc1jVQUl9tYJqoYRyWYM/FMK2/Xk89dpyDBQM9pWkJgmwiCHMOk7aeNSWJgQMChe96U07O3tQGMjCp1pY8Oz9iEXpovs5EngH5RkuEyQ2XRyDI5JFulmfn3Nq5ni9xaJo4/jQ3bkX/fkydm9ajZYjzxyMtMK43UK3y1YK2EzG6+D1eQuxYOVOJFuaUNfUyAV20pF6UkfBIjtsuF7E5RYz2YbPtnDXzFa0NjcgNeE4VCp+LF0wHx9/vAbb+8qoqFGGoQTNqfZaJYG76eCZ+3/O8r6LfnzbIISSub9TkGEE8/lC2DaSYRWtsoEjp47Avo5+zFmynZ0T9YN6qICCKUUkyqGI9PM0s9Tw7UUpLyrQavgUkatFImE0NqQYriYScSSjIaTqUtxumYzFEIvFOHWIxeO8JtTU4VeE9JMdEkdwj+Bh+o6dA8H1bDqNluYWbPp0N554+jms3bAJDl1Ho4o7br8N27ZswquvvIyWBNXgqZ9Y1GoDPoEk+HjdmjStH7XwCQZYlCJFLyzQNZBHUTOYEP1o/vOQjLLYI16KQa2mBkX7koAKnsqo1nBrIm4tS1RruLSOdP7CoE109ORx/o1PcJ3eg/EWCBWpWP7cjzFuygxYviiMcoEbTTyZI+nl6UFk72AmSzmuLerTtQ/vfL2f/bcMd/+KPxEi4YdR1bFly3a8N28Bxo87DKPHjMawMRPw47teQqYE7vUkqSCdGBluMBxhY5aIbeacC5xzkLpp3/79fMA/Ou9YXHX5RXxBFDrhWqxu2kxsMJqxLCa+iBn2hyJQqNRUU+fyOEASDGzctAlrly3BUedezJMRmMgRtQpeOIKqBJmZpLIZ2GAgncGvH/pPxBobkWhqYQEGl7gIiioSZJUWlcK38PIcDchIZBM+W8JdRE61tSA1fgZKZRnL3p+LVavXYvuABiuU4IkOTAgZhhg4YFl4bNYtUEwDt9z3Z/RkM5AUHxziCwjNUsC1BFtvwIRP0jCtPogjp4xGb7aC5978EJIpwxcQm5PzYArBlN9S1CASjjeX2OS80VwJn5fzeaQdfab+Vc6YiQ+QHS7JGIZGrS01yjgfrx0Zu991xuxguEtM9GgHaQiBP4D6ZB3O+9oX8bVzzuXOrY/WbMQtd97HnUiU85KTvv7a72HHp9vw1uzZaEs1MO/Bx2I7/Pqe06RrRpvZg5W1ZKYjK9AtG129GU47Rgxvxtt/+Q0qJSAW9rP80/V+zN6S4bLc09Wcc7p1SOViMBi4TfC1RkTOgpvyGShLeOHV9/Gn11cy289+jI6VCSwdq1/5ORomnspcTyWbHyTwWPOgqLy3KXhw6Yd18Ac3FXhOdojfGGLHBc8zdGR8LWt+IA1seM5hNlbXUcxX8MxTL6OxoRnDRo/EmLZhqGuIY9GmDtz3xDuQFIJGAi4TbCZZoUyazlCAWUm6EMzYOQ727t3LTm101MHsJ+8REccRF0hAWfrWRrlY4uhBzoCen8lkEIklEIxEWEzheUPKYfkhAYvnz0NfxwFMOfVcFCkMeVDfERCRPjzDJa9Ji05tgNf/8hFE6pvQMKwN4UgMikr5uegM8vJIoVl2F4zgNxmu5eCu81oxavQIxMYdDa2iYvG8d/HhilXY3l+BE61zZXyUU5vCcG0Hs356FUa3NOOPL8/BstWrYMsqVEtlgo9guUGmJ6vQTAthWcdRDXFMmDiCHeRDz/+Dtdgh0vZSzsk1bTFKiNIL2XZQJa0vORzSWrmdVmy07ugfzyD4Z27nDDszlrDSMAoS0IhrQamDQQKYwcYSV3BB6YtM4htBlDGh5xKTV1xyAa64+Js8fGDhh6sx68E/uq14JGJx8Iv/uBaLFy7C/LlzUReOIEC6c76MDqgRj5w+oQeueXKaReIGKsWJJhbarDROSTMsdPWmWc134vHT8dSD16NUMhBx94zYFg5LTNlQXMP1Jmx4hisMxW2i9wQbNVZL78f1cR5mQCN1HPz0zpexbEs7p5GDdWbLxtknjsHDv/wWkqNPZMKwSow3iXWIq3GlkGS4hMC8CHuIQGvwnQ8yyEMY5IOjMPE2LvLJbX2BySnabO+8+Q5UuQ51qTo0NNbDFwpg82cHcP8zc1G1FDhU5yRvTOof9kwRhBMxzsHIyOgARA0W6O7u5oVsifrw9K+u5KjI9UNipSUgGo3xpIlqucJCDhLMMyFB+YbqQyQaRyQWH4zQg4YLB8uWLMa6lcsx4+RTobSOdw2XAyRffJ6+4ZJUJPRnHbRZxX/85gk4RFANH44wvb9LFFHvKpdEXEb7nwzXBu76agtGjhmBxPhjoFf9WPju21i9ai229pdhBOJQJUIPYjIIQWXdsPGTb38dMyaPRyZbQUNTM9K9adh5TdSMKSKo1DoWgOyXIUdCiPooT7aglUrY2UNCBgtVU6AHypUo18vl85xH9/TleLJEe0+/iMLcpO2q0hiSDbW4MZrynCVbjnAAzE37RF02m80w++1FQYLBXjeKKgvikDckOW8yLknCz677ASaMaMPEw8finQUf4uGnX4SP5bEW/LKD6665DCsWLMHyZUsQ9QX4fD1HEXAFCpSymIYQt3qkIh2PcPBMx6GiG+jtz3EU+/bFM3HzNTNR1g0WdXgEHO2bcqkoXqPGcAUUo2d5wp/Pr9+y8R9quKaG83/0IPZnqCwn1pgexN4/8ZuLcNYpM6A2jGGZq1UlfbkhpJL0jrKCSrksGHhP5lgb2mu+/l8Zbn778w7pL++5/wW8/e4KDBsxAsNHDceo4cNxoLMf+3uK2NbeCVtW+KIodAFcrSoVmSPxGM9v8gfDorOGk3qHHUFPdzeSQQkfPHsPbMliVRItABmKbFqsaiKpXDAYQi6bY8KDapBkzOTZQ3XxQXKKYBLlN8Qi9nbux89vuRNnnDAV4864EIZFr0ksJHlKmwk2ryzkko28TE+/8Ddsas+jeVgbQvEEvx9BP4uQgNuT662ngDZMSPLgr/vPH4GRo4YhMeEYWEYY8956Ax+vXoGt3QbMcCM3mlN5SjZp7EwVti5h5qnH4vvnX4AVb6yAUwoCVZlzZtpcZCB0Tixo55IHnR8RQRThCOoR/Ddg+2zOP4WWmPo7FQSDVJ5z4A8HEIyFEUiFsD+Txe33PIS8prNEj6SlXFvnHI+rbKJBnZwas/Ui33JkEdm8/lJO9bnrRaAdzxnTurBTptKd4/Da3XHzDTj6iIkMHd+evwRP/OVVhtMUxJsSUXz11OlY+/HH2LB2PYJcTpShGzpHVR/X60UE95AaiVeYnPTQFaVQZABVA725PA8l/OOsn+L0Lxwp8uRAYIgDsSwUC0U3PxZSVeq59R4eKTXYDcQ0sxuBuaVU5J5iOJxIOyi9+MJl93KrKOfhruHSMS5+7mqMnzIDUrAeWqHE50TP4sDE7fsSpx2i1Hew0MJzEt7hfR6z/S9sfPDHUvXT55y5763Ev9/2AoupKUeh1q2pkw9HS0s90vkC1mzeD43ADeWDPClClDaUQICVSKQLDoQifNG8aXZ0pvv374Nk6Vjy1z8ipGgiMfdOQhKb1svHPAhAhMoQC1fjHW1R5qHSzorly3Hdzb/FT751Oo6d+R2Y/DomLEkIKMhw6XUJ/hNbyR0dkoRVn2zCy2+vQF1bC5INjbzIPJrHJ5RankzNg3MEKemYKZreM3MYWtqa0DjpOJhGBAvmvoOVHy7Fp/02KoEUyztpjpJtUS23jEkjm3HzpZdh3RvbAY2YclETpjYh0oYzqefIfHykt5Vk6h7REQ7T0DOFCTUOiyYpcUSDB8kYaepAMhV1yxIWSw2jagRGtIopZxyFWY8/g4+27WSBfG03CoEKWj/elK7x0eant6G1EnBSEEJ8XWzRTMAbj8tFYs8QLPSuz32/+jnK2T5MnTIZr89diL+/+wEjCVru8SNacfnXT8Pzz7yET7dtd6cdSowcOGq5wgpKkYiNp23BbLw0NErHF6TyGJAt0IA9mthoYuHrT6AhKdrtvPRGnJOFQp5KQaJ0WGu43kA4z0AEXBaKO36+a7i0CNFIlH9GFQq6Zid88ze8LqTY8gw97lex5C8/Qtv40+D4fKikxXyp2mkX5JQ5fXHX1tM+1BqpZ7i15NihxNW/MmBp2Su3OFde9yDyGimEZCYe2lobcMrRk3iwmq364QvH8dr7a9BbKHGbmOclZV+Ap0n4AoIkYMKHciDyzI6Dgf5+lkGed8LhuO36K+AjscQgoyY2iPA+okDueSLvYD3HK57nMXE22tv34BvfvAbTx7Xhmlt+BZ17dkm44P6lI+qAJOwW8Fv0QqYzRcx69BWE6+rRNLyNaXuewkc1atfzC9gp4JXQVVPwMznitrQ2oXHKcTC1MFYuXYxFC+ZhR7+Dii/J4nMGfJaEEfUR3Pbti/HRq7tgFkUOGQj6xEhP+nAlo0Q8eudNAwQo76Q6L11sPmYaWkDjarlPlyZOAtEYjZMFR1yCspSn+ijXI8Y1KWPy2VPx7VvvwYBG8sCh+UbE6guyina5KMsI4cOQ4MTLY4XAwpW2shELldbQtRLr/PA9v0ZDjByNjRf+/hYWrFrLLXqaZmHG1HE4dnwTZv99Dtr3HWBDpbDvGS5BbZYzqpRiiYkSwjG7cJRQCKES20auUEKupENyNHyy6BVItu6W1Ya2NeWTNCBOMLT/O8Ol4yFy1TPcVWs34fr732HeghpYvP35hSOH47l7L0F8xKlcS9bpfWlAn6dFIHmrSeo1IumGorln+IP72/3if2W4k+plJ1bXgC9+4Rg4RgnTp00k14yq6SBXtWlOAwb6s+guaDyKdOeefWxwXLLx+ZmcolojDdCicgIzj/4Q1wdtW0NfewciUgVvPv8gE0FM8HMvgVvXPUQV4m0e3l9eXZFgGsE+0gvQTCgHWLhkCSKxJvitPIxYC0945KYFd6Eo36CckDuEXM9Hxv+TXzwEX2Mbho8YjmA4yOdBPoGIEq/vWLDUohyiSQ58hom7LzoMI5rqUTftJOiVANZ+9BEWzn8T2/pMlH0pvgQ0toZkfU/+8iZ8/NxWaBoxzIQ0bC6zcOSndjIvV/IJFpfbJCUbdXV17pwkMQ1C6GIN1j+LlkMH8XgMlk11VAWBEMEym6NDPBbj802NjmDBgd14fv57sG0xVpSWmssr7tpQV5qAx+I9BvNaYtTd60ENDExCsx5UuDF+rivYp/N9+sFZcHSaNAG8+tpbkEJ+TrF6OjswvDGJpvoEfn//b5FnKEkbW+FZw/Q63JVFY13IoN3ha8KovZxQ1JlpDwxkcihrxIWo+Gj+02wQYkqlkImSsWpahT9c6onhA0NlrwTEsF8Qp0OBwav1iqBAxBR1X9GDHP3jL76J1xbsQKFcAKwAbNlkNv61h67FscdMgD85Fk5Fh6bTNXZ4TJD30Fwya8i1eNLcg37C3zDicaW7tbCaf1ejiqwNbtKcP1ztkGiaCu0GVNauHujoga7ZKJky9nb2oaw7rKSq2DTWRjBn9EGGq6gBxIJ+qEEFpxw1FVde+k2ESSjg2AhbNBhbiMp9chWmFOA+U8mnwMewzGVwCeKSQoa6gOhCuJGBUz3RwgKLSjMUIcgzWxYWLFqAYWOmYNeH8zDsuLOhSTSYusYDmyayuRzDZc9Tkme/7Z4nUA7GMWLkaFAHCJezaLIjf/YQgDsilORq1MZoO7j3orFoa0iiftoXYBphrF25EgveewObe6ooqUneQCSPu/obZyHVIyP7qYlSucqCAsMUxkuOiyINPTjHNbwoJiEeCXInlBeNvc1D5JpHuCXjMU4JyJ0GAz6efEnMeLVSQoqN3kSmUsLEfzsa377pTuhOCTppi60AoBK7Keqi7nivwfzVy8Pcyq1YRMo/XRGBt6qsK3bHzNC1ePHRB2BrJRSLZWzftBWG5GDNqtVYvGQRfnv3HQgHZNx5xywUCmVGNz6/yoorehApRVM0BFkl1EZUyqFUyHuwZlxR0dPXD003MWXiSLz69F3Mi4TDBGlpWJs324wcgilKYm4XEIsuXMOlTb9h/TpMm3bEQWUVNg4XzRGxJMnuPClbwm33PI61e3X0pwfAzs6h62di9as3oXX8VEi+ZlRI8OEesme4jPZchOIZJn3mFKTWbt0KL5eL3K//leHWlvj4er36++87FhtjgJVi5Dn27e6AIUnoyVXQmymhL51Dpmqhq68Cw5U4EsQhsqohGcEDt/07Jg9vwd63lwArt8Ha1wt/XueezwANOKeD9lE+R80lshj9SkO8KJ+iIrwfMGmjBP2QkwnIflUoelQHKs2Goo9kDJFTj4D/xEkw+srYsHktwnWjsP69VzDpnEsZFnq5G60NeW+PiRWmT9vDwux5q/Hemk1oGzGKFUgEjRSfYDC9uVre2tJikkMIeIbbmELd1BNg6mFs/PhjLHhvDnamHfRVfUKcDgOP3HwjPvnLVlRKVGKzWMNt2SROFwNzPWUWXUSv3jxy5EhUCrlBgTvls94xm6YYek5N/HpViOdlVTjPaJTywypSdcnBUgV1Ek09ZxLmrpiD9dv3Y8n2PiarPJKJ2dqaAfRetBUbuGYSBXEQg/ppsSJkFKyTdpveX/rjA7D1Mk+szAwMoKOrk88zFg6jpS4KSyvil7fP4rtJ0GtRbu85K1p3ym+pU4rgMR0Hiyeo1cF1oMQ/6DbQl0nD0B185/Kv4hfXfpMHG0YOMdx8ITvUEfQvDJfSD683t9Z+PMOlVk8aLEc5r20pePiZv2Lemg4eAqFTSc5S0NIUxBtPXoPh40+GLIdRztH7esMlxFBFRnsui+8FDe/9/p8Z7uyHrnXIQ9BG4EWVVOzZdwCmRcJuDbmygWLFRJpu79GZRbEsBpEFVBUTxw7HCw/fgX1Pv4ny3xahmVhTy4JORjkIwQTsYxKopuOfvCNdZN44rs5YnKSASsK7C29Kt5fgMpSiwnfTv+HTrn6EfQ4yMw5D+7r1GDZlBhNUVCIgppE2vUZif53GwIioxqUMy0KuVMHb7y+FJgW4XzUQDKNAYgYSRih+FsE7sg+qTBuUDIhezcZvvzkWTfVRNE05EbZUh/WrV2DJe+8gmQihLpnk3tipRx2PHSvzyO2qwqLSEOU5VCs1RR5JkNbP6guX3TVNtLQ0CSTh2Oxo+JYo7JldNVu5xHJH2uRapcxaZuqljYSo3kjGX0HbyGZRBnFhV3B4ECt2LcTuvQfwzpo96Ncs+AjNhEOIRxJC8caQkGCP28pI8kFXqebVK72OILIjFnCwkIPKLQ6CqowXH3mAO2b6+vtQyOYRjkaQyWZQLlcxpq0J+YF2/OK2X0ORKbISchDQnPy2SlDf7+e/p3Wn1ITOn3N5cuZUEqJJoLaEvv40qo6DR2b9BF8+7Rh2eMGggMrMHtLAwkKW0wbBJAvz8FhxL+p58s9ao6WrSyiSrg8TU44Kw67wbO47H/or2vsr2LW/B5aj8nD1S75yLG7/0SmoG3MG5+Ua1W9twfyzU3RJtiFmXPSY/1cPdqo1TvJfTcPwXoMj7mtkuG4uyPS17EOpoqE/W4AkB1Ck5vqSxl0fNB7m48274TgBtKYCeOflx7Duhvswav2AgIPEvhEb546uZKke3cbD1aSqzpDQgVQ7NNWQ8z2X5fS8E0FKEmnwybh9v2yQkoRqQxSNc+7GppN/BPX2i4Axw5Hfvxtm8yguVYjiuchnaCN4zdqstWV9LDD71ddw5umn8t0HaPRJKOjjMo1m0R0GDOzsSGPSxAmY++EaaHKUZr3jwUsnobkuiuYpJ8FEEhvWrMSKRfMR9pNEzo94LIkTjzsHi17cDVu3eRC7ZwB0dwOumxKB4U7tp6maw0eMEPCONrM7eYGcZ5SYZWKp3aFq3NRNqYJOUjtKFQzWLVO0bWigCRWWmG9EghFqUE/5YLSZWL1yKd5euA4b9w3wZPdwUMW3vnwKlrz7Ks784pfwyYEBZKsO9FAYCo0gqelh5fUSN1Pi82eGlCWJVHqTEPH78Owf7uc17unpYeecLxTQ1d2Nhx55BM/+6VHk+vbhF7feCdumqZQElwNsUrTfAm5XD527lyKwcMaVzYpyM017BPr6M5xivf7sA5h8+HCXlRe3BiGWm4cdVopC6+TCYxaqHHrLm8EykyjveA9voiRBd3pNmvl1oL0X9z35Jj7d14dcmaoT1J0r49kHvoPTTjwCgYYpMGhyC6Eq13Dp9Qi91g49F4TgP5eDatllrmbUPudz8tpDI7f0/KzLxSBb1iJTKUblG2gRPCYIoWkmjwwp6TqyeQ37enqQyxmY/dxDwOLVCPz5A5gEAWkEDTUp0NhN13N7hjsoYXNv6ET9jjwS1VXI0KoMlYAczjW5W4T6GrmGKYkB5pA5V4r+6UbseOlNZHr7EPjFldi//D00nXAW3yFALIjDBundqMzzvASVaNPdcsvPccIJx2PSpMPF/Ct/kEtgsWgQYWJ/HQV2tYiySZMdbGanT5/Wgrpk3DXcBDas+Qhrli/CivXb4Jg6vnPxZbD3R5DeJ6Zc8M3PPPUPRXSXLaVxK4Q+6urrheCdWt34njlDk0VMQ0MoFEChkEddHT1PRBVTozUTs7CIzIKkI5GMIOgXih+WDdo+FJw8Wk9qwfxF89DbX8Vjf5mHlrY6nHPSDMx56SWG64c3xlDvDyHZ1gC1uQmfFVR8mqEZxUIn7m0URkS0nu45UeHMr0i47gdX47ipdFcGEz09vdi1ZzdHm/vuvZcVXS8/+yTSvfvwy9tmQYy1IqcllHVkoH6/mJfNyIxHBymMSLgk5DLZPAbVtJGjMo9s4aN5LyEcIsmoGBzvGS7fQ6laEvk3BQ33TgS1UY73xb8wXO6G4vsECRRChjd37hK8OG8j9nVmeFwxlaLojhMfzv4ZRh52JJxQGyoDNClTnINXU6Zq7v8Xw33lge+x4Yq8hXprxaym3nQO5SqVJGQUylWkswXIaoA1t+OGjcANV16GjsvvR7RiQyGFC3kaunuBIyLloMzLrft5bCVtANq4NLOYWU0yWpe1pIgkanOiBhbwk5TSHSlDdxzg+wYpSI9MYuLDt2Ddt29F7398Ax2fzMek2LoysAAAIABJREFUf7uKo43nyUhKRyIQik7UIUQRi2vQEnDnXb9DV15HXVMTR8CGRAz18SCSYYVvp0JN33UN9UiFowjTqBufgekTGpGIh9B8xMmw7QQ2rluDNSsXY9G6nShYPjzz61ux7m/dKBXLyJDTc7tQ2Ou7JVkel2LbSKXqWHBBtURyWNyd5IjeUxHZ6H44VdTVpcRgM3dig2hXFvmqblSQSoTgUwzWM5N6jYYDyLaN3lIZU86fgtmvv4RSuYx0sYot6z/D5s072KHQrVbaImGMTcV4cuaxXzoV7819F62NIxBuGY0NPT1or1AUUOD4ZKh0fUg3yt1TfvzsB5cj6VMwceokVj319vUxYqVzpTbNx558Cj+/+QYM9O3HnXfcC10n0YmQ/nksNZ83OW5XhEIbn/6eBBqeSILSpnK1yudAfMmmxX/lu2IQt1JL4hBTTQ0G5JQFiVMjruD+X1doUSv+rY24js2pCDsPEn0YOq6//XGs20OTN0WLKBXkaDTQ/Jd+hpbDz2SupjxAY3CH6rfEy/C0i0Nu3FVLDR+EAtzIKhx3zQG5XWMC4g9pGWoHWEh/++1VDrfEmeT5qa7mZ8Pt6s1y5KAhbDQXuT+b45IPlQN+c/vt2HjHn9DywU6YpHnlOaokCxNpB99gxKt7eY3i3GcpciVSp4joKHILL+IO1hm5Id5AmObluvI3rrdS2YRQgQ00Ln4YC069CvPVAdjTG3Hh1TdCc6EdvTcZiSB/dJEHsXqI2GMHn2zYiuf/PhfR+ibEUg2CuabJiQrBOIdvSiXRBShloCgmjhnbgu9fdBbqUjE0H3ESbDuJjevXYM2Kxfh0XzdOO/NsNJfqkN6pIJ8roFwSrX2skHLvS8T5tmEgHokxk025aTIZ5+dwq5/bZsdyTa2M+oY6Lp2EgwICewIVT95I+W00TPet0aD6RcSgzRcJBtGRLmL6t6bjuRcfxrixI3HLLb+FZft5YgjladFQGHU+H844+WjUtdRjf1c7OnbvQ8L2s6abjC+YiOPEiy7Gg6/MQzAURdhvY1RbIy788uloqY9C8ScwbORoXlO63SfZBMP8aASf7dzNDrF/oBsPP/QIHJvu9Eh3InRvRObuUS+F4uvqTj6hurSQPorNpBni9qWQqti46G9s2AG/qLXSg9YhmyVmlyg3t7zDrYuuJfDGHyrBHZpriroveE9yDm8RJ2Pi4usfxq7OLAcOErLQq/3HFWfh6kvP4NuMUJ+uWaSJk2Ltee9SfuuKfw5ihz8naWUU+N8w3EHKuqb1mt/v5fu+6/BoSy5TUKRUeeGyuQqqVBCn4rthIpMvolQ1MXnSWJzzxTORu+Be+Gn2DhkJyfP4s3gb2k6DD8/w3FGuRDTxIGxvzpNruLzQrsaWNi+RNNQB4w2sE2NT6bYaVHpSoc76Hna/+yFy23aj9ZEfYv3WPWgdNmJwSh95cjYe8uDuhAUSB5BEngaSjB03fLB5W6ObSeUK6M6W0NWdRldfBnu7+pGvVvkeMOefNAbnHjMKsViYDde04ti2eT1Wf7gIAUfCzAvOx5IX9kIrUBsXOQshuqCITw/asMSYUjtkJBgWEZSaHywDca59i6Mi50kbNx4VZZ5KpczrRPCVmFeqkVPkoteiOzqQzFNyKpAUMaKUcmES3g+UTEyaOQVXXn0F7rj1CqSifnSmy5g7bzXmv7+SeYgff/+7aO/eyY6G4N7WjVuRCIYRsiU0NTdg5NGHY/WWTxGoH43DRzYhEbIQRBWth02H7I/yPXubxxzG150MlwYIUB6bzmQwefIkrF+/ETt3bscbc+YMGi6thefQyWF7hjuIOujKMMnmZm+OhAoNNzctHHf8EXjmtz/jyZWkba9FdMQXsO/9XxouGSbde5mOg27fSRNGv/6jPyBfpuFwpA2gY7Uw+/fX4Jijj0CgfiLKxPBXqTQ3ZLgUlYX665Ce2/+HhkuWRXeZlF598FpupKc3oy4M2lQ0y4dCfpXuuseEEzGeOuh2nHfedgc+/vHvkPz4AE8CIHtj76HSd7X26pIbjsxMH32QekbIzWjciuhYGRwOxtIzMUCO2GfOrWoWgEem0hj0ACm5AnDO/wKkyeOw91ePY/z8h7Fk3SdIJhvEAdAxU47Jt9uk+7WIIWRC8yGc1D333I+jjp6Ok086Hg11CTTWJ1FXnxDsNwlFJBkawSTLwc6dW9EYqqIhlUDLEV+Aoddh+9Z1WL1yPoaNHoV4cSz6t1aRzZdFlGe45E53cNMB8mU08pNgqjhEGv0pBAGJRIJvjE2GTvXkFN2ylG+aJoyUYCRFFoL65XKBG0AYurqN5o5ThuqTEI8HEY0m0ZfRMe3iqbjm2h/jsDFNOPfLJ6AhKSPATRVRZLJVbNu6DTv3tKOvP8tD4j7dvoenbM78ytlwAg727tmBq666ENt2tKOkUeuljVR9MyLJVoTCCVSrJkYfPpmhPbVxljWhWuKvCwUcaN+PbZs2Ycvm7dCp0lDVuT3PKyV58lIBB4dKTN6m9/gBru3aDh741TU490snoFrSWdsucnBxl4F8IS+kmO72qyV+vNzW4z4+rxxE+zYaoRo5NTU4mLt4DX7z6LvMNg8y7ABWvfwTjJh8HORwI0okc3Tfj3TbTGqR2o3aVGv6bcV+d8VGh7TmHSSo+JyWv1qozOvi1oJFxL33KjEBgzYKTwChhmQaOGawbEvcmYzIFgmJRArf/NJMtF94F2waRVozlsNWRH7JCh0XpQjqX4Wf5zKTzlnh16U3pp5Nd6KS2MjEDjJcF1MXPCUJRyx3tArDKVlCOBZGaVwbmm7/HrZf9ksc9tjN2Ez3EyIn4d48igdeGyaKxQJveu735fooMc90v9ddKJbL2L51G49E0S3SvgYgwxT3DQqqmDZlIk6ZNh5/fOJpzLrpSjQ3pDBs+inQ9Th2bN2MtauX4vwLv4Flz+xFrreEStXkcyAvLfS34jYbDPdpNCmL4l1JHzU4KIpotKZzClJUtZBKxQdrpXSlquREDZ2b3akcFKF7tsrkBN2eYZ6aaBAlgngyiFisDgMZE0dcPBnfvfpqKJKFyy69iG9mXd8Q5FG4VIMncQSlPnmN7ujXiAULluGEk0/Axg2foLuvG3FVxxdPGEN3H8KBjjzau/qRaBwPNZhAQ0MzO+ymEaPYwZKx0qhUijYEZTPpAaxe8xHynb3YuHkr3+FBqw6Vg7xI6+X0XsSla13bm0vPo3SBHvNeewwtjUGYBh2vN2mSFFNVvpuBUOQdXCUV9wcWZsOTNEXB7J8EGCStJGfgkYWPvfgPvPTOBkZF3iMOA0te+wnaJn0JUMIopbOD+mRvj5Y1ocOujbiC63DFF4ccn2e4h+qTa2G21wLLebB7D2H++qW7r+S2Pmb73JDJ0xFNaimjmh01lBNDClxwwYXofOQt1C38DDrlIq5HooM16Z633niaGsMllVmMJt7R0bu1XVG3GpoEIFg4TzNLKllvSBqJ/N082O2fpIhLA7H1VAL1L9+ODedcj8SFZ0O+9DR0D4hiOF0fJr54lAz1xgqxN9s0T3OUEY/IaGtOusSYmJ5Bf5PJVZDO5LFp41b059I4bGQb/vzim3j+nmvQ3JBE27STYZhx7NiyFeEAsGdNHunPLKRzFaJAxYA6Zkf/D2vvAaZpWV6Pn6/X6X1mK2xhC8tSpCpNECkaRIiKKGpECEaTGFvswW6MiUaNvUTUGA3EgoogVXqRXVjY3ndnd/p8vb+/65z7eWaHDf5y/f/X7/PyYnd25pvvfd/nee77Pvc5567Okfp1QoZpZ2uSNz4Bps8Uk3MkChcf9aukLcqczpcRJC0Qqa+yHdFET5eZk0s2x7GjAmPYTuFxVEY6E0Z7Wx+mcy2sfc0qvOb1b0YrKOOyV1yGJYsXorMtivZsm2h7nekU0tl2RJKdQDiLeqiGZtWECZzAMDP6LKKFHRrSzLGos9UwxvPtGtZGVgkdL3sXLlHGwJqYLUQvp8zlpnHfA/cht/sANu/cgUKDtEBGbYciO902Nyb/L2TZtQx9EOF7Mf1n+s1rvP+2byOTpjcV+eVHjMHp4czD4k9tXLYIvcPin9q4HOotzrTQ8xre8nf/iKf3GxjnX9dceDw+9u7LkV50EoJGHNVC0Y1PcYMD6EzqpkL8v9y4mmPsAUy3cXXYf++mNyriCjmjEXeViCbnzhjTh1pWCr4TkTje+JprsO3PbkK8bJpXOdITTSYSKmd892JYd9pY/lwqEhNYpAfFDyHp3xEfKv4b00Iflf2pK8DfnTSKlVqknMERRSQbw/BvPo/Hzn87mh0pLP3Jx/HQkxvQ1dNv6bDT5Jar3LhszPOhW7pNjPCpDU/h/ocfxdmnrsXKFcegr7sDwwP9yKSSqFFTWq1g4zNbUC7PYt3q1Qg18+jMJDCy9iw0Wl04sHcvGjPAhtv2oVys2jDtqi1e/g4PRrGu5QHCF+VgbOewbJBDZjyqw6RULmHB8JD8kxlRBfTxMGUJ0mxq8bLO7ci2SeqXTFEfax4NYn9HCMxwpEkL3b19mKrVsOrCU3D1tdci3hHBxZdcgHQ8joHBfoyMDGrIeCKRFuHC6249+OWf/9jOBxCrjavGIb2QQpJqPYotB1tohNpxzHHLNN6kt7dfzp78OZFMmk3kCtMoju/ELT/7DfaMTgrc1CesmyeTRSXvV2aHz/ya1QcSUmp17dEQ7vvVv2jTUoTBA8Be5jEldJ4JqaslSRDxLUBRIqVNdlxheWs9v6+aITDFz84MslHD+W+8CYVGCKEmJ/MZ+v/Aj96PJccMItK1As2CaaT5rlEHlHnRvI+4z4/99mntoLXfPT+d9z8zF63n/bA3kfNtOZJTcrOzCH3rI1dr45oEyfSbQv9cjUV9bDVo4lWvuAKJ+3eg8tXfolzhsOqWLFcIHinyOlsSF/BslksohAy9mWnpwtS4BbFlJMTWyA9nq8oeYcvpK90GF6+TrQJ/ErOdIB1wBIloEvG2BAZ+83ncdcENiNbqOOHBr+MXv74DI4sWO8M/A6c0woMR3cnnWAs+/dSTeHb7dmzYM4njj1uJbCqJamEaq5cMYO2Kxdg4VsepKwdQZe3UKGKyGGDl0gH0ZuNYuO5MlMpJjO+dwYENeezeMIoarVnrAaanJ+eQZInznVuFZ+yQaMD0K0GATTrcCBrNGrq6utTKKJeL6t+ypBDKzxS/0cTM9AxGFow4ZRFRaLPaoVuj2mkRWoXS2qaB3v4+NDmlYVEPPvrJT2Dk2AGcfuaLsHb1Wov4PDCj1NqagyafA58/a+tcLq9NRET/0NbfIlKn/WkYyWQW1GLICxsxHJyOonvxaeju61Imtn379rk+KNfR4Z2PoDM+gV0Hm/i3798ubWpUm9D0snq2nPLoDmXeE3HfSXF06LsypGhcAN2CgR784gc3CYPpbOtA1fX9mYTRUZIZCEOB5y2bx7IbSSLFljNadwHK00l9nCFH2Ud6thbOvOp9qJEp1YqK/94KSnjsJ+/HwjUnI5TsQok+TgoqvOfmeOqHVv/fNq5tWPutz0Odj/r70a0h/71+MAFLE23cud5SyBrkmprt5nmSh3rM4mNwxZVXYfMVNyFxMI9yhDR3jdIzxY53p3cnmZQ1gdmhhOsEYQIEZAxxwyLkRNQEpqxtxF6ZqXNss1oqaVHba0G5+Yg0c1GlYmkk2xPo/eVn8ftXvxvZyRyO/f4HsTcGlDkpQJC86TvpFkG1E69ndO927N+9C3fe9RDOOvN0TWmgFLGcJjlhDdKNaTQD0h3LSKbiKFcpK2vg0FQZq5f0oTsTxcDKU/DcxlkUt7eQH6/g8MEpcGod20iVWlHSMtb+vB7W5MpmXJSx4VQ0SuNwZx5CQAeBKKlDGGHJ260jJZaYWfLQRYGqIbUbdMDVEI4Ekglq0gLR5gR7rsyLqiDvOdTfiX2FGRSbdSxdvQixBEn8hkgbG8oOQLHaHNWO6b1F2zqmp6dQ3H8vx32pHKBgX44VkhE20azk0X7shagkB+R8snXrVr0v21FMmw/veACHJ2Zw2gWvwdo1qzA4vEBYSaRhJRmvSxFOuAPlfkckfWSzsa7l8+PUP94bfvZjFmVRJZ+8JQs/A/doMkh2XIuHc1VMOO7XeqWEajGvsqXZpJj9+fFPQWWeoES2SS7D2bx9N66/6WaUajzsSSwKY2Aggd999Xr0rXopmmHSHE24ImN4d//oejL/PV8o4v6/2Li8Z3KO/M7HrtHG1eZl6sshRw1LPfggOX/0pLUnYnVyBOUP3IwCpVPhEKpEbclJ5hnujjAPIvHWZhNJoau68X6AsenEjEUTtsl4Qu2YsGmh+ka5a09pELmrizgtLm5NegNzsuj+wXtx/zv+CalDU0i94XzEr3gJDu4dg1YbT0oynypFjO7biX079+LB+x/FqaefiGUjWVSaKUw1ouiMtHDuRWcgGy9jyzM7EImnFfXa0hFUa0ChWcIdm7vwjj8/C0G1iR2PHEZ9KoI8J9FXgWKpigpBiQCoFHJz4BRjgJElzMmCC1GqKkaXaEz96I62jO6B0HUnvZODR7lk8j2SUFJ0Z3JSSNrjCHmvIx0nfZAHBAkSvCf8piqGhxei54xj8ehdz6J/ZSfifWkkmeqKceVSSPc8dLAgsFm3bEXVyzg0MYG9G+9DWyyHRCyJRNJ46VznTOtJ8avUm+heeQFqsS75aG3e+Chy4/tQL09r0PSrX38jhkaOweiuWVSmSqiXWwgaYSTCSQcSATVmbeQ/Wx9HBxEPEpZcYs0xatJ1UzOrbAazZYYE/VxfWzArwTb+n7RrJ1GMRhBLcqRpCBEePHTWFFehhuLMKAq5GTRKBi6RgJXiemlGNIPqi9/5OW69Z7MkmUrqQ3Vc/bK1+Id3X4u2hSehUamgXLaNKwsn53c2f+OKduvCuaXE89qj7utHR1wf/Y+Oxv77+F+uHw6RV6bCGtejwwTD6bzATgM3pdDRRh03/PW7cfDyT6I8OmGm300OZnD6xjDlbNbw9myYGNs54pG63N6hajYo2kHjpInF4oqOCTGirKbWAcKmN6ODU13we+gvNIe+hUNoT7Uh8aXr8dQX/gPRzXvRXLcIa778Hjzw8BPIUGGEFg7v24Otz23CHb/9LS6+5CL0t8WRbx8GFq3D7c8extKggPddPIxYiDV2BZs27UGUJIZ0CskUS4YYRpaegFhyKWrUunYPIRxJINQyMrwUILocuyamv6qtXKtCaKZzYWRWIeaXAqlzkaCG2PppcyNLXTFk0yO4aOmNWaphfHQc+zbsxaFdh5CtAbVWHQnqiNlWUx+9iXC0jmUnnoCR01fhrp88hMWn9KOSILMqjUajMufQQNM1LgJ+1q7OTul9efJs27oZDzzwAFr5fThlzSJZtCayUSREkifzDPLLLlXr6Ft9EZqJbokAHrn/12gWD0jBc/3ffBj7dszi0MYZhMoxmbrFIgnEogm0Yuxx2qTCZp0m61XDNgIudIIwIsJqHXBTZ2iUJ+6xH89iYBEzKfWB4zHZBbFDwVKDmQxrYvbGs9k0SpWCEytwsmAOQbKEdGcYi45bjL5Fbdi+8THEawXEU3EBs8RrXnfjp7Fnqq55b7RbCocS+P7n3oALLngJQulhFKa54Q3V9mWcNyb0m2+OSDS3eY9syxfasEf3fefXv/77eRhQUTU+Pm4jbpkqe2dEblxGXDOlNqeGNWvWYH3bEoy/7WuohWtqEXF4JS+S6CKlefyzr5OZdoQbHIdxhMblp5dJRO6dLlwkFuLqmE1e6eE3rgqoUEh1sU/ptEVcxE1+8W3Y+NVbENm4E6GuLJbfchMeeuAJNMINHNy1HXfcdjtefNrJGBjuFEmkmBzCg6FVSCfDKI4fxKcv6EQiYY6J9InavWtSiHMknsWy1evQO7QS5UID44encHj3DMKtjJz0GXmYlgXse7vDlAswVDEBPr/Eg4douVwe7Bh1BAu2TCylo6GYvJeUOpo3NR9QNmNDuwXShKugq3UoHsbgwi4MrBxGOEjh6Z88hqlDo5oyoEjVaiLbHsPQCauAgSy23XMAx5zRi1y4hFYoiliUtaWz0E1nlG7RhJ7kiWwmo7bUX739HTjp1HUY7O3HxN6NOO+01UhlNULc/KF4knLj1uoYWncpCi2qfkJ45rHbUchN4Lrr34MdOw7gwKMB6rPMMmKIJzkegrUr3TzswOJC5zrh1AFNwZCYgCouIpos11rIZGn9a4wrDz4RByFZhPeUG5seZELwJcYgDbQmmihpsfVa1cayhO2ASkVjKNXKRvmkk2PvBE695HTM5HehNXtIffFys4lXXPtJ5Ko0g6dpQ0ssugf/691YfNwZCCIdyE9OIuxYXv9/Nu4LtYDmDvIXiMZz9S1bqAHU3hRH++sfulpjNj2STPiZtSajZritDW99/Zvx4OUfRv9YFWUO9Q0a0qgSU+OLaTLBKaKfYrQwySYfmYvQiQV4E3giakKd5CG2uAVUaSaa+RboQzohtUcWiTSL7ujkfiZcCCGRzKDna+/C/f/0HXRs2o9qGFj/u8/j0c3P4cdf/yZGFgxh7TFDWhCToTZsjS/BWGoY/ZkqTurKoK01g/VdeRndNcNRKW9K5SaaQRYrjj8NhXyAJ+7eiWY5jmSQRTJK07KyIoD/TLwU7+Mk0MWl+joI2f4IkRTRpl6sH0rFQ0pqGA0Kt4jryfY8LAlUkQ7Jr6kH7HqWjteGYpBDrDOMky9ah5n903jqJ3cp6nJywPpzTkPn8Utx/2+eQKsUQd/6djRTVHwRjmiJWcWDktzzvr5+/W4DxUr45Kc+IVLGmtXHY8XKFRgcHMTeHRtw0vJ2tCeJS8RkYkcTOtIQB9ZehUaUHtoFbHnyTrz4nAvR33ssHrh1G0JFNwhOPttpM4j39rFaNJR5RrV5D48ddqbvtBsS4VkHisz+3ARGmRQ4RhXvC1NUlnEkPtAhRL5ijYZkebzn5KdzQ+vQ9JMfKQ/NsvVWNgAwEUE9lsOLXnk8xkafQZ3jQWeKeNkNXxDhwzyom+iORXDHTz6AoZXniAtQIoAXCsReYp7N0sZrjL0HwP9oBx0ln1fsOYqk8UKRmBuVpRS/l8+N4KE32At9+X1XBfkCJVGqpFwqA4TjCbz+DdeidNcmFD/yY9RpoK1ZKnVUgiZqPI3omsHZn0ELiSgjp9ViVGjw3eYG/BJVZBokiVgY9UoVWfZ2XfQNmnWxlXSvnG8sN65O5mTK+nxOZmZ1CaV0WQz998dx719+Coldh+Vn9MiKOFrr+rBquButekH1y2TbSvyu0oMgkkF/OoorhktItKYxsmBYn5uACXW5zAZqzXYsWXkidm+ZwdaHJxEPEmKRifwgIoQNreZnNA0zU/2q3TkN3wqLqcVoy4g8ODik+lcnqrdYEXKcVirsWVSMsvTnGh4Z0kMi+urJCfwvFzEXinjg4SjqdeZGBay+cJmMCh7+7s/R1tWGkbPWItXXiQ2/26nIMnBSL0LtDVTqVZvQ4JhoKSmh2sxxolHRDCRGP1r5DAwMoVgsoVQsI9PZhf+6+WZc97oXY+FQCrGALpxllGsVLDj5GlSDMPYeOIzKxG688rLX4g8/34RosQtTM9OWlgvDOJJteDCK94MHGw8SbsDZHDnhZpFLbTP71myRzecyc+MKvHSjZmy9UOJY0+8hMkx3UOv/0kPM7GR9RFd0VvvGPLzYimPWkRho4awrTsOOZ36DbdsP4C8+/E2Hu9iOeN2lJ+Gjf/s6tC04AdViGZViSZx2yhI1b5FtR41OsbzghV5HGI82GfKFXkdvXMtgW4hHzR2T94Ke457aGvrSe66aG2wtIUsQYMGCBbjqytdg9y8fQuXzv0S4WBYPuchZIZzFE4ZQ5fkblxvS17UaHiKKoYnHaRKn9JLIKf1wqf+UCNqRwnVCBjYJ0NW53KyefM8Tle+p3J4pJ10gkiks/cO/4t4L34n2XFluE5lLlmPy5Da1UHhIFDIj2BJbiH2zUVRTKRzfHsKFg6PoiqYRontEKY96JIUo+UHNLBYvPwObN41j15MVxOnWWGPmEHIjNG3TKhJyKnqCdVtMOmSypJQ5hAJtVG7c4cEhM+d2TB2zPJUd4ZEeYxh6H24a1mVqkRklfq7eTyWSSmN57eZ6yHlABiiVG2WcdsUa/OG2u7F8aAiDJ6/AH371OIJiQkDMglM70cxQUxdIqmhtmADt2YxcHSbGJyQG2Llzp4gqmQytUt2w8loZPZ09+Mb3foBzzjoFs4f34KLzT0BAMghaGFl/NSrNAFt378FLT1+P3c/mMfF0AzFwYqD5dHNyIfvFVrMypbeFLvFFyAzQLdMiQ6wsVRb/3ffxGXG9nlrtaqeMkiFBzAQRsrVNJPRMiMlYKspWkrH1zB0zhnQ6g1yBEcs5PLoh6mwFHvfKxQjFpvDFL34B37rl0SMbNwC+/Ilr8KqLz0couxBT4xPKquZvXIFSDmT9U4L5uUkTDoQ8OuIeDUhpDbjsjbiJ16ITmCI+0NPTjdC//M3lQaVUAZdYR7oNl1x5Ffomm9j0jzcjtYXeUzU0WpYYS/3QMgd+3nKf/un0m0fnkku9NquG3ZieViMOzU+XD0fTRwlaOSKab0kxCul7mSI47ylRvTiPxonr+Tniqxah55sfwtbz3yn0mLDFeHcdnTecIiBmJ3pxqG05ikELhXoCK3szuGgxhxGTwUPheVS+WqEwD400+oaOl3vjY78aBWdV2pxdI6aoZcUSwpl4+2xCEYQaWDXjAY4rpTXr8PCw0nn6RstbqkHXCjOCZy+OAArbLpwLxDRWEr6uDkUfLbzA1CqKtGSJ1ex3mzyR2s8kIrR3pd9UuIizrj4VpYkxbNk0huJuShmt5ZJclkMrxjQ9QDbZgUjcrGjp7HF4bEKLvrszi/EDBzBLhU+oimxbO9raOtRZYLP/jxuewvihcaxYuRLReB0pjcoMsO6Cq9UJHCBIAAAgAElEQVQymZmewmknnIG7/v0pRBspgZoh9toTcYyPT6hdxA3EqMQD1RBiUwlxbXlQjwuSm4ByT4/K8qDXuhC4GTWXlgZlf+zvGwmDmYW8tJwzpt+4mk6hEbCGkZgtEbM4Z41LJls8pjWFTAtnXrMeZ7zkbOybkHjYDuJoDPd8751YftK5CIXimJmeNhFNxAziuUZZNhjZwzJB/3p+BHXdE/fPR9JkI58cDU7Nj8g+TZZE1Q20Y5kT+sxfXhqEolG8/GUXY0FXP7Z88gfIPnEAiLG9URJqR40tdYdawMT/ND7DFrTAJdUtR6RTcdbIRN48b5OFPp35aMjmUmEvPPDjNv2HZZ3X2dY+N3PFEnjrmc3d0FAU3R98ExpL+rHv+s8beMOJ6h1RhG5chkIrid80jkU51g+EGzilK44Ll9MKLySHBdY4HBAtCh5bK23HoqtrBX73H88g3ezQw+Tm8iNQdPKLJGCgiGbUOuN3Xg8JKeoNIkBfX49NDXRRmJvWxlJwIcXQ5JAzDTQzJ0GK5tnL9SMuuPDoDOIXhr/H7A8zmvO9bJxLSDY4QTSBkRd1ITWcxnP/vQNNKoYcQr/otFGEMtMAUmiGqkhEF+PAnho279yp6fW7dm1Dd3saixYtlJa6LUtKJQ/hMA6PHsbuXU+jWi5icjKHgYEBtHdmZLNZyE/jFdf8lVojy1Yci8d+uxWV3TGZqzPzSZEt1uLIy5yMGFiTGnvNi9RscBkPJj5XZmDcyOxZlwp5JNlXdb1e3Sj18zm3iOJ7+mZXnUtkTPU5D1jzFPRjVRtKhXmfaErnN69lR3Xpodkvnxu3GY7hhCuX4ovf+Ta+9u3vuh5zC7FGHU/c/gn0H3uuDO/JWOIr7twcuaY5YcOCjnWXj46e8xFiW7+OeDLPLfOFIq7/mth2kTDGxsYlmeTfOzs7ENp730+DdCaLrR/7LhKPbEfAcQrxGKLsJ7YaKIUDzX5Viurm0BKv4wf2PFOdmvOkSxoxxGkFvi/bbBmpgIQNN6uGIBYXszyC3Ga2E9R0uCKHa2atG6I9r5iPdLZj0Z1fxYOX/TXaxnKgElgT5RIxzFzei4cGT8CziVWoVetEvpCuTuLCkRZOXpxGF3unjiLHeB8JJ9C7aD0ev2MclYNEP81VkadxscjhXdY3thnABKNs4zI6yhSedjq0gG21xCUmMOLBJ14Pa15mJNzAFBkImJE1KRddWUZvZFzRelSCeicwn9u4jv5otkIhtLe1G72QJu41m3JYQA4X3XgB7v7GH/QZJUrnwh86jJ7hHrR1pBTBSRlsNCM4PHEQd999L/bu3YXwzKSM87bt34cgTAM3G6FB293ObAsz41MYXrhIRu2DA0Pyj56amsAp57wSmWQCQ0OL8Pt/30YTSW2uNGcAhSKqH3mdowcP6cASycH1bU27S+F7RAcRa1NGHn7G/OyMwCZ1J3g/2G5sNJFMWDuwWiObyyYYWDZk9Fu2lqjx1s+xBEnSe8zsivje9LYiqNTb06PNG43xWVuGw2fYd0oGQ6tH8PEPvFeHAUe9DA924UMffiO6+46XXJMHC78/6e6RDPfnlE1cVV4PfIR+8T9BJ2c4f9Sk+T/VJlJLMBwSHsHrZ7Yl7fDjb7ouaN2xUYN6a7WyNgwL+UqNIzUomaE3Ygi1SADKhllnJTvbEe7IIDLQhXR/N2Ld7Yj3dAmsaRJYODyB2uPbMPHYs8iQjsaUpUrChiBl45UKKWa/17ntuIgtNJoqHl27m+cTCSPWDKEWbtIJHCt+9yXsuv1BlP/lZ3pPotriWUeB8RdncNeZr8e2mTriLT6YCBqoacpBfnIUo1u2Ij27F6evW45Tl/Tj5DPPxvFLT8bjvxxVRKsVCTqZCwgXlmeqJOOM0uZIyDRQIzUpgo+GFTm4YJgGcwFp0gPvm4EGQq40zZ10zqgza+fw62RMvTljLFUE1nChOeWfO73JeGqoDibSq1Nehx9TXqbzYYQTCSw/rxfP/nE/GhOMygROmug8Lo+Jwqz6uByhOjDYi7vuvN/8nQHs3rMb9cIE+jvasW+sgqo2SgTFUlmeWSesGsHCRUMY6O038If65MIspmfyOO+yq7BwZBjbHx7FxA4rb1hrClGvtnRNqs3CIYwdHtN/6YU8xyHmMvfuIPPMAhltZ2dmnJrK0Gmqd/yMIf6X78FDQUZ8bnCZzdYN0CZdrY0B5YHBTUy9LjcpTfdsdpUNPVOZ4xVunU2cfc2peO97341GuagM6MY3nouVJ52JSKIbs9Mzc4eFNz7nNTbny/H0TNxIl3kg1PxRKKZ0cbFX5aOjP7qRKEfSZJskwetkn533ngc761tluRte8cYgTOJ2bxtiw4PILh5Ez4oliA/0IKDUjNGJ2A0RPBb21SKSDoXNlUuIFmuoT+UskhIFI2gz0I9IbwfC6QRq20ex7X3/itkNWxBiZCKn2QZEauNycr3YRWwhEYBxHj6+leRPoiDKTR7F4q++D5W+Lmy5+iNIShroke0AzWgNtXOX4K6zLkYykcGuXXsw1TmM3Ng4cvkKipNjQKWIanEGqWgYX3n3m3D6iSuw4fdTKB+MolTNIxqwjmqIoSKLnURC/UHR3yJEdFl32onPGoosJ95QooyVkknQBMTQSJ2UT5dS8+ustZjCsfZltO2l/pe0OWY3NTeaIx6VD5ZSMpdicuFx4xAp9TU3nRrIGKpV+VwiCHdWccqlL8J9P7wPcW3cFtqX7kI9xujSoUl3iXgffvGL2xGJBqIVHjp8CDu3P4flxx6LHXsnEGVUk79xSZ/vjJOX46KXX6CevDjfrQAHDh7G/Q8+gnf+7XuwbtUJuO+H29CohUWW4EHH961XWcuaZJGZBaOd3RPLKNQCc7OMtZHmAZK8l8YQmhE6LL02HSBr1TmXCsM/vJuGcQj4d66neCImuirza1Mr2ZA1yva4eZUdaoKCpaCMvk0iJJEAZ71hPV77xrfg6ac3IBEK8Kuffhgr1p1HiY2ki8pEvP0OiSBcz/Ook36UibKBeYPc/yTpQmCVi8BCadyGdoeBzZ6mCQM9o61t2Nvbq4MsVNz8aBAlW6reQLFZRf3gJMoHJ1A8cACNfeOo7h8HihW01YFEyShq/H5uVHoReeYo0UQ9DGkDNSQIhZ4U+j53PZLrj0PjqX3Ycd0/IL9/FNVIC9GggYBEDbGJGGEtFQ3XW9b/dRpcAiSKvuEIlvzb+1BdMoznXvV+pAnkiDUUYUmmGTitSAuVpXFEb3gdJlKduPWJLVgzMoRFmRB+eu8T6FlwHPYf3I/JqSl85f3XYXEb0DuwDA/8ZBtaxThK9QpSkagE9IV83vTBjiEjLnHDVCxWo9oCZI3KTaVIosmAPO2jQpsZidOufuMjYQuG7QsuaAJYQdMDGxYhuGjzhZy0uXygXtbGRc/+rlEnnS9XiykkQas4CuUmcuVJXPjOF+O+7z6MRDylmvxg7RFUgxksXdSD3p42pNo68atfPif8gqNhxsZpdhbg8cefRM/QYkVlCk34+fp7evHRv79RSp9GPauv0VvqmWeekoHex2/6JA7tmsahh+toxlqyzJEEjwPf8pZ1SCpaNwEBN7TfuGrvhUyJxsORm5cAH1+WxlKvTTKLlWjcvKQt8n5KJSN02uSZYvjxz37gnEa5BhpPyvfnUG/+Pg2Uc9MgmQQJT9U8ZANRYqE4ll3Sj/FaEa969RXoSSVxy83vw9IV58mMPed0wb6zwc86f+Nqs7oZODqc5m1cX+ce3bv1I9TtGv9nes2Ny2ucnc3NXXdfX5+yr9Dm5ecHbOVIhkeYnWJ02qW6KQJmim3oHm+yRyy9IZbvzVH87j+gDUI2rx660U8tG8Sx3/kAKody2Pu6j2Ls8G5EeMCQVyYbbsrd/HR2MmysnURieoI1SiSMVT/6LGYSUWy55mNIVmpiO/Fw0Oeg6RiF+OEmKovacOjCfpSDFEIa38ETNYJnn9uCVjSFBWtOxFvf8lY0y3l09XZgz7NFTGwMoU5fI9rHuBSYD51/N9UH38FNfRd7xxYlI65GPc61tawtxAdBAMWnYhQFsC4hH5cnd09Pj5kJcNE5/2iJpVyflWZxdnABhWJOp6zIGCQhubqfMct8p4FimdMRSzjzTevw8F0bER5voRkJMHBSGxBnCkneNr2CiyiVCxJS8M/ymZ6ZwMMPP4zp6SJyRdqj1rFm1XJce81VQCihNLNcsYHRBw4ewMaNTyKIxPHtr38Td/5gE2qzTWTiaYGXMqCnVRCZd26MCwlRfmqdoq7v73O4tu9E8P46je6R7kJ07h4yc+Gztt6mn8hgBxjRaCmaOKZlbjoElWZxgX6Msha5jcQhQoZYpm5Gs+u/xmMhtC1I4ZTXn4Qbr74SSxd248Z3vBEdXcv1zMj8EnCo6Y4WGXmQNI8yjffPf370nNsXR1navFAk9lHdZ1xcg7OzU4jH0+jKtiOZjeOhDbsR2jF8WsDFwyI7iETF9+RN0DR417f0fsg+AglPcnUSf5YEhQa9drxDvktd+MsF3bdCKHTEseTXn0e9Auy+9K8xeviAicrZD9aUPWvUk3qmjciNQWL1QD/W/eJzmNl6CLuv/wLitYrSdvPCptmtsd/VjkED09kQUu86G/UgpgiIUAxVEtejcRy/9hSk27tQD0Kq45YvW4E7b96K+rTV2easT1vXqk1m10gQWr2S8eVsNx1pnAuIG6pSKllaywdaqwosUvrbNO9gno6U4VGXq9qLM3Gdo6GiJ9tjIrAcsUTlkEaf1hnQktT9MGGPmyCvU9oECoVKE7VyE8klUQwtH8LuB3cp/Rs+sQu1cFnti6Y40lZ/hee57BNTqFTLeOLxpzA6ehjFagV/dtnL0dffi3yRQ9PIC45q3vETTzyBZ595Gu/54AfQmx7G5jundEBX8iWNDNXcqGQK+ZzNOubhVGYpxSgqK16boKgxqxK0WNRUNtM0b2hLr4lC26FuYF3UKLbOHI4/M3dYzpPqcREoisfCstvl2iJmIMojPcyc95g8qmWfaxE3FqO6KowgHcZLr3sR/ur6t+Kay0/C6eddgFC8R1MayKbSQeHUVUqx2XP+Xzau750fqV2PpMPzI7A/sOan4irTaPlTt4O8Fs3gKz/bhOem2xDaNHgqoTlBRIlsB0qFgknOPKWRBueudmWNZrpdLmZyROviuYrVMs9Amy0Spot68eTl/ygY7+/C8t98AWP3/hG7bviUhOPynvDDmIhcq94Io0p0dvkCnHvLv2L/rQ+h+PF/l5skHwQfojG0WmjwwYQ5cc82SzEWIPb3F6LElhRqKAchdLZ1Y/W6U6SxTCTbtFAr1Tz6+hbh3u8fkvsEGUnarLG4alAeUlxk0sSSxVUlFdQWAaMDCRMiELgDTO0Od9AZsmuTzRmpIhGjdJL4bv5E5NUSfY45uR0JCXa7VHuFjcBgabeBLKI8ztu4/s/8mVKtiaCWwN7pvXjVuy7DAzffJx/g933hvWhGK1h3/Hq85JyX4OSTT9Z8XSL3/sXowc1pw78bGlxGOI9Dy1PpNswWZlDO0ySgomvJFwt43TWvxUO37kYwDkSSEURaURwYPYS2bFYHmEdguVa4cf3MIhkpcGJfqaxaX1lZk1pic7rgywM//C8jJn+n7oNvB2p2kaXUtnkt+2HGxAjY0c5h6GYazx6hGG0uvfZsNNswFvG1sUI1RIMkamHgnL9Yjb+4/m34zHsvxaKVZ6IepDA9NeUAR9u4foC6aLn/y8Y9OgL7++5/99Eb2m9cHlgqMXj9AL720434Y24QEwViDTWENnSvD7hYSMNTTUKrlFodcaF2lk54l3XeALoh8KbJPqMVCBVVGu34lJ5v6rWJfuSmasBICIX1S7Hi5n/Aczd+Hodu+TXyTdZIDeRCdfSduRb1YwZQ6+7A488+g4995gvY/a1fIvjOb1AVS8Z8/MyTwOSE9Le1ifI6JTR4KvyBl6EQM08rpn46rYMYCvkiDk1MIZuK4uVXvgm18Qx2PEI9px1EPIHN59ec9326It6sSBhmcs62j48MjOp+M9shZK6MjIRcpNygpBiydh0c7AOtVkj+kEWN7HCNtxximeKmETACcWAZWxeK6AS6KN+LeajyiIsgf54G5PVGAuNTo7jk7efgnlseIrUNn/n+J1Co0eOZEc0irmcrEcEmJ3jJ0iVYuHARli9bhsULF6BaLQlA7O/tRyrbrnp/cuIQanXWcFAv94Tlp+Cem59BiCNA3QAvZmjjY5OqBz2SzoyIf9dBzpTWfXylxUqpbRN6Cx4PXGktsiSRQZo1ctm+4cNXhBb32owN+bM8ZEkHnNMtN41ooXZT3AlmJK90UdNlhp5Qw94+sZZWDDj9qlX47V0/x0vWZDCw7Cz16GlGJyKEk/ERSfb8ZIa8uZcfseMMAvzX5+t0j96oL7Rx+TZJSr8QxbPbD+PLv9qHg6UU8jVzRVHb8I+dJwRMdRX2nfu+indnpanUSu/uepmIIJPNGlDA044pjecoz/NAtjEgNj6YPTW9PxUiyRjav3gjMievw8NnvgWPlHZiwaWnIL16BPlwHcVcXS4Df/6612Pff9yN2uf+U35INqjKUqRQJCTnQHF3xY6x/IDyLk4wr73ueNSWdYKGKV6Zw0lqXALcSATCzv+za3H3Tw8gyMclVayWbVwJf4f5TBs1T3B8rarygWkw02PtAvV0G+q/8iESoCIyLKoneboBLWksarK9RNUKwaVyqaJoEwoZ19lHEppwC+yS2VxNhAfxo5kFxNkHroi6d2Riu/GfmU6VK1Xkck1Um02cdtVabNu0HcXDOdz6wI+Rr+VQKZeM3FAqKWJUa7w2ShkbqDWcOL7JSGtYBqmHf3nD27Dm+HW4+977VAotPfYY/e41x6/GjgcmUdlPIs6RXj5XSblECx8TSIgHnEza3x1ZXlMYnTCeRAulwSIYmK2PbWKTryl1pl0OBRoaMm1kH2mUE2wT2SHEDIxAIidDSPDh3Vy43pzxAIejKdWUHJCoNYOSbXrNIpYIhusqitXnD6N9aQaNyWfQ1rcMM7PUWFuGoo2rWUMmO7RQcaTv4109ZBTgkGGTeBpngRf4pxDmuU3OSEvmYTyKJ3fN4gu37sXBSgwtMtmcvluQ8PaFZwWMND6q+NrBi9z5ht7T2Gh3JiDgQiUB2tP0vCujTjFnJcn3ogiBvFoxkfhQIiGMpcM47tF/x6Z//B5a/U3kO6pItqLIizAODCxchf7+lRg97+0oRo1iGW858MrdFCmSeFNIkVTeaF5SzWYY+XOHUDttRHVdXIO9OHzZmvH8fyiUwDkXvwl33rwPKQTIF4l90EW/rtYF6zRuRn9PRHiI2Exg1V8y8HKDoV3tleXh1zCvLhFTGk2UikWBeb29PYoYrOt40wnvc96Q0mKJ1MMInCkY0de2bHqu9mUNyujMdJuR0JcgfjI8a+RymbOKmogk4lh85iDqrQp2PrkFO2Y2YqY8Nec6yefC66rUawJcKGzIFUwEoXSTwFzdOgepWBRtnV3YuWePWKvMXLhhHnv8Gdx/8xNIVJJoeHsescZ4qIZxaPSwFrgGeCkVNbYcRRfqx8aYFpcRi9hnkRjdWeYSwPOkHgM2LYVmfcznpvqVLUNHVmHtx03d092tDMhHRf4uvg8R7UJxRlGaNa7MDqoVYRlkonET8XdywwUtHrpJBL0VvPQNZ6M8sQHRZI8GmvGpqU3lNq7cT53BocwU3ctvXPVyj+xEy1r9YID5fV+vTXcBT+HRIcy/uHsnbn4iQEnG+mSlMYjYgAAZL2wbeXHg3eOPuOVTQGH8WHvNS0c1IdMkYr4RLsBhvumzZqtyFoy1dhjFuAnsQ4WM/H3Tteh62ZnYeONNKFzcp5lFjN5M+84470o89fpPILNv3JRGfGj6PHZqeU2vlTimnOAG4FZmWlw8phOhN58oK1JuFt5QZhNEYnlyvejsl6JcGMT2PxTN/5h80ybrIjvVuFisbLAHZEJzoKOjXRuP9SgXjBBOhwXIM+lIJiu6H/9dM1c5ST6bUdpGDrT3VmK0tihqtbOJEoBEzJm/sw/sFwWBnWZFogePQPvnUy5xQTY1d7htcRrDJw/juTufRiW7Xy6PRO+pKOLi5rUVCXhUqjqomLlYthVgZnpWYBrTwzotgFjr03OMNXCliVe97rV4yxvejg237tF9YMuDP2eZSRy52YIimqmOSDYxm12+uEnpq81SRBvQtXh4nxhd5C3teq8G2BkPXNarLlJZL5jP1MQwjMw017Nsy4wX5jJAx0BjqcFnxfKEG5iqI6HDySPOjmxTMbKr5xxUcfHfnI1qbidCkTjGxsYUxeNzRg4hOVZKoupagnMbd95UvheqYedHWz9EfW7Xa5hACPFwGN+77Snc9kwUJXCOFdc3cRG2FNxUBQavrSNn6dbyhPSsD90cpgNucpolzs4lj7rGpM1Z8SkB0zVK9bzJHL/XR27eXJmTs8XkjOi44Gb6M1h255fx5Gs+htClAyjEq6iXa4hnO7B2/YXYd8nfafFYP4yxVMN7TT/nUi6lzrx9Gi1CtQijRhOz/XGk30V+KQ8Ja5moppRWs4WXvuqNePiX46iNRWWA3ar7mTVO9+lGPnpvZAm7nY2qiFBCZ+0UjbvBZb5u44LgK5+flSKFBwY/G+1R6FAoET1PcEZS0hmDBhJxo8vxACToVasWHUHAeGWemM90sVIqggB0nGCca6fUG4xGtpFqyQrOuvoMPPZfD6PRvR+hSF2icrW2NPLTDiOPX9Dojv9GJL3WYFupLHF9IV9GKpm2A7FZx8x0Hh/9zKex94kyigfokUUFFrMB6/tycRFDkClIKIR8IW/SPi1u1pwcVGZaaoJ/Att0CDclJ/REFAMIY2JK8XkzQs6NJ5GayGYpMVK3yd6HaqmW2H5ztq1UshWZ4em3S3lktrgGRumQndNEM7BwwqOVNASeTvzzY5HoqKGSm7H+c5j4gqXJfLFuFxg5X1MrEc6RfXIk4DqXEx8C5xE25iv8WFLSNfPff70Bv34mjCJsrcTTZNORLWYZpR8eF9rYc3LA09AMoW0atxA3OeVruzqswT4A00XaWTINlOxOobuFbJL2KO6CONfU1QDeBI4nlOxbHMLXjAJDt34K9VAE93zpn5Bbau917LK16GyNYPz6T6AZNXI6HfbpRuBPLA9iPH/jUulBW506RqNVjHz6KiGkRCzllhCn1I0E+G6ccM6rcdf3n0a4FEFZg7isxmIbQ3QyotsyzQtEVGA08MwZ/hvfkwudJzSjH69JIojACAdMq9mOYOQiP1nc23QCcQIsLomSGUA0JtCKKCgpkh2dBnoFjaqzuXFSSXGlWQ5w1CZnzNuEO3+qRyIJ1BsRFMoVVCJlnH/92bjn+3cjMjCGZst41Hx/z77hVEU9Zc5oKpbVj6a/FFF7L7tT31JZQFP0R0ocb3j33+H+bz+HUDMhk3v2Ejgnie/L665UicQbWMfsoVwqI+nQdT4rblzrf8esNUPVUlsG5ZpxwnkPueG5oNva2sWA8tRTH42pIGrvaDO+tiR7jpghpxRuSOvTckPzuUh258zluL6Zdstt05Vclm14bjTvdxQDZ2Sx7JQFGN21RQe06vK4Hch8sa999MbVWpy3Keei8FEDwPxmt5T3iKVxKBTDfRt24yt3TKPcjCOIJBFTOUXTQmarRGts6IAyjyc7Tgj4ZppNE2f9YD001miG+pl3lOeYdrV3GE3Mp8H+w1Ijqj4oVTd2sZ4RI6GAH1btEDf++8xZK7HiK3+Pu6+4EUuvO0tCx2imE7nxMCbe83lw5LIALtYMtGadP/xXd8YAGlvUNiqF59JMpIWRz74GuSb1oLSBsUHJBHrWvvjlKE6lsfn3OQdImSRLvGOe2hHblKQ5cm4Q74e1dBghOZg6JldFLgJ+tpT4sG6siJvVyo3O+iuRsJaHShlXm8TiVtsxE/HaXKavRHipWJLXstg/bqj2PMCPN7ZWLStdZtS39w6bfVCLA5lt0PXZf/ki/P4/7kHQNqrIrFlznE3sRlkq13QvZlpGBpkHqBCwcUbiPGBKhSLOvOQyFEaTGHsir5q3QsM0URxJj6yq1ODGK+TN5ZKbiuQNuqIoGsq5xMAskUkCAmt2MDPSsW8tRZUiY0htHbqtGLBjBgV8ETnmNbJONiMCo5YqC3LtNJ/t6WASVdM2LJ+HodUWea1OBcLRiLILcYJCYWSHozjpVauxZ9vGudrUYwsqoZy5ok3Pc/fS9+vm7qwLe0fVtM9Ll2WPQ8JTA+OFMt7/9WcwjTY0YmnZvsaTaStnahzknVLGJC44p2Q81XWiM0Q3obv6Zx0dRn9zhm1EgxkxbWK32/FuQfkPwtOUp6IMy3kCayMwzXKsK9/2IJWP/rlM26IxDD/0Zez53I8w/qP/Rq1Vw8hrX4bCypWY/dBXbFzHESbY8yKubrxQYEvNvCkbb2YhEmDBh16J8SS9mDlBwMjvTCXPufw63HXzZgTTxkGm7pSfm6AUr52pNFMjfj91yjwRGAUZOVWXiLFF83i2j5pIa7KCcZe5CZi+8cAiwkzrVxMb2CEoml7UDjQtGNIDqUHVbCACfexvhpFgy0N1HdNJ+zPbavx3Rnv2q9lOESOI1y7taBLleoB6pYYX33g6fvuT2xFvnxQophaPi/TKkhzZRC09j37O+R3bBvYHN593pqcPp5/zMjz2090ojfMwS2rDMjctFug6QbUUyRpGCzWBe0g4yMThMRC447rm16391ZKUL58v6B5ZKm12M6xV+Tv5M1QCMRvgvWPKOtA/oFRZ6bHsd6lAMvDR9RVMyOEGirFNVMznRBflIVcu0zzO+uG85zyQxZVWORZGPEWqaAiteBHnv/VM7N35lK7DJKVO/0uket7oy/llpGM8Wp463+rC39v/8XWKM0KoBjV86N/uw9ZiP0LRhCyBSBhiek5ar9cQM4Mayi8AACAASURBVHD4/n7o8bbj3dawMYEecu8d6AOn2NFipCWWiKUTNr3MwJP5LA/Pu+SHZiriN7hpR63Z7Qd8MdqwtmLU7vmPD6KeTmP3pe9CuVZE6sozkDjxJBz84JcYQp8XZeenygIH3M2xtMXqRG6uYqiF2DUnAauHEYmF0ag1JIfqX3wshpedgSd+fACVotVdOmxicbUU+F9+RhqU8XSjAIK1kjX8WYvGEecM4ahNQVdLQYivqYh4f7gQWA8z/ybwwtm1mjQrX2PycMNSCvH3UnjPeyiuc5P6XLaEmggHpmG1iGoRhx+CRAmZYmtUhqWkXLg8kCKRpAzDOe7mhNevxR2/vAPDi8M4dOggkhzWrXLAMhih2O6/RsQ3FFbAm1hJtBgy2ilbOC+5/Br88ZcbkKkM4sCBQ2g1w2hv78DefYY4c/FyNhDbJpp84eieau3EEyLaGE/btMncJnK6cACWrF8jvNcFpBJsz9nmdbOrVfszI1HpIVDpyNgSUj0ZIFLCFpyxvxu0RrklLXA9+433T6YG6qNz/ZgjBwk/as0RJ6HzZrSC8647DQf2PWMjXnTY2cYV8eN5UfVIXfv/eePyXYMWfnH/JvzwwQaq4QSiqR5UmUlyJAoZhRHXVmU22QwELioDfaxjrVJlnbIOWPC6UD5cwuWkM1LELP4ua0K3YTwyxp8X7d59nYIFRh72Dr1PkC1A9z38PhEammicuwpL/u0juP/E1yA8PYP0Jacifcm52P6OTyFBL2JWdPOr+KNSETvdDF22YhySHx5a2YYlbz5P/s+ZNDWsJZxz+TV4/M5DKOyIiNHj60RNkBdgI4K247Ia+ql6goAK5XrqmyaRlIuE/TsF1lwwMioLM12kqZqRBIRiFktO0sfNwe9rU8bBk7PWrGGQ/Vqi8qRxOiYQf5cxpgi6HfldHVk7OOXCILsX6wmrhaLISxQ6jBUvX4oHHn8M0ehhbRIt+LR5J/u02DOUGHXmUNu6SRB5bcl4Gs2ghjMuvgxTO8vIbyG63kJxhuBVXiwpjprMF8qoVQmaMOMwcYGuwx0MJP9zo9EZhP1gblBD43nomEujPzQUTWS1aoZwJflzWUTm/3VfWTK5mUMei2C05+EkVRVxAL2HqYy4BvnyrC2NQdGAbluLyniSJlAnZkGhCbW/p752Ncan96NSG0cmQ8TbXprV67IXre0/6Xrxv6fKvE/8/X/9z/dgMjKCZrwDkWQbYikzDPC8eR0YPBQ5z6vsNOKPd/iIy2fmhNw6fY1Lyovv6+5BoViw2oSppXcnEDrqDMtdW0ZjMmUGzlMsKtXR3CnvLt4saQI0edGpOIbv/Fds+dx3Ubz5NjRWLkD7e6/F1jd/CMkghBjra3kWz+uXebraUTWv5ztXwsD+jhqOed8VCBJhJIMoIp1dOPn0V+DJ2yaRHy2iWm0iN5szBNNZXwpwopF7vaE2BFsE8xk87GfrnrA/rAFeBHNo5Ba3dNctBuMTOyvSRl1ZC9s+BFvk1FGyOpAiek5akPqFcj5FWRN80J2SiziRosVOzSRt/JqrRTV9SYveAT5kXcFqxkUvGcFMq4idW+7X93PR0ZXCz/eZnx7z+0WcbzblgMHPxgxgejaHk847D6F6Gvv/MIFIPSHTuVYthG3bdittbYU4gnQXopGEEHxrCxGoi9mfmeaqN0y9ctLRLW0DMt0XAUL6VcMMZLimdLklVNk2vVFRBeD5WtlpWg1INEsfIueWNFgLju8ld01xvK1lqM3A9l7NLHI8QhuX8ZuNFCEQ19HWg0Uv7kX7ghRmcns1cdIfEqZimseWcp9Fh59b38+PyPbF+dkp/+4Pt3/+3u/w0P5O1OMdCGe6EEtl5iZ88B1Z2xPxVgChgUOFf28h9Ejb6sDXUX7jGo/TtTvicaGfczYf9L2RiMAr+e1jegIGHwSlbGYcHAicmGs/zAOoGEWJTIrc/433IGhPYsuV78Z0q4Ghb30Qm1/3fqTnNi51u4xiBkZoRIpP1d1dkvLPAQTVoIWpZB0LPvpq1Dl1oQJc8qa34rHf70NuWwSVnOmCebLu3LVThT+nnIvW6HymvDO9IZRUBxlARy4uox2vV6AK7T7TSUOsUwkdxroHHIfpwA5mLGQv8exhROSIjwUjI4rKjIZKT1kvp5lq07mBdTEPPJYTbIdERCAgiOFVWWzHqD+udkkY8XQalQp7vTUMnDSEjmP68Mh9P7FIQ9Sb7RWX9YjcMEdpZWpL8zue8lb/cqEsWbUG/YvW4sDt21GpxFDImWEdSRbbtuxCe0eHShOiypOTMwIAdUjI8tV6+Hz+smGlY4WqbE9RJJLvNhR7Ww4f4PuzfGCqPDw0JE41gSebD2TPXGmrR9ndIC0Dy1ivRtDRYS0i9qNVwpDdRkxBLUT7/VxG1YoRghTN5VkFHTSck8T+P4arOOeqc7Bj15M24REUY3BihVbakbxv3sb1KPH8+bj+G5+/ce2zTE7n8defvRulbC+iySHEO3oQTqTkq+XZWsQseD28JyySWDaICPpY+1pRoYSMuk3ATcpThjeSi4kDovUglJPbtxmiduSliepO4cHL8ubbjFKsaZliqLZxvUfJ+Pyg31ecjp4Pvhlbz34rytN5xL/0Djx04ycxVA+QDMJymHy+K8SR3+3TPP9J9LCCAGORBvrf83IUExFc+sYbsWdzGeV9wPjeaZRmK4riTDX52fI5yt2sXzjf8Iv9OuPb1sQlNufAqA4RXn+jWlebhwuMt49kACO/N5Ei4YLvx1kvmixvaHKj2kBnZ7tmACnFdQtSelJuQIrtOTLDeQlzCh+7SBwh4iWbirp8RhRjiBLJGpqzY81Ct2tJB5acuxz33v4ztLdnMDY+qgXPQ0GIrwO1rN6k+39R94F1KOvyxWuPx4LFq7Htrl2IluOoV62VNDtDA3Nayc6qFqQgpFLiPNy8XE7URZiHgTDWx2XH49a72kQlJFPcyA6s0wRHZiFFHXgExej04QeS0xHD/L8ccUezhoydxmyF7SYjuqS12AlAGYWXkk6T+lk5ZWNMxCngoPZy3oz2SfaAlYTm11xGOJpANZHDy996MXbu24QIsQcX/US6cIezJknOYz/N7YZ5GamPrnPMKR7dQQQ1FPH+z96CHaXFaKQ7kWrrRiKTpZWh8ebFt7Y51fy83LBSvIt33kLo0bY1AReAPoAmk5nxFT8db4D6qM7sjQuGkUX1kRM4z31YZ6XJn+F8VR8RWf36ekfpgbtQcoz5+/igC11JLL//G/jjyW9BtJxD+IPX4OEf/QLdG3chQ1mRU8b4lMPD/fNTEJ+O8waRZjlD5PDqM3HBh/8WhcMRjG2tojLZwNRYDqV8WVRJ/n5DM9lTY9O+qEXNjapF5IyxCckTxWUNZKQLDgbjTB2SPuhRZaATWxncAOIic8GyHUGgq16FbFZLrHfTKBbzyGTpF30kjWMPkveG70WKKP/Mz9Pf34NKuYAoxeHsSTtpmmHJHnCiEiYudlS2pxvVSBVrL1+Lu371X2gFRW1wwzCIskfmNq5q2WTWMopwBFXW4/1DOP3sl2HTHc8iXWhHhZMWNfeX0+Zz+r6JiRkd7FR9FQrcPBmMTdA10iOwbuCb0n5D7bmB1FJEQ77RJPHMIa+thq6V6DyRaNXicqkwxp0FFjusxQtw3lwUshcLeSxZskQOHbn8rNJrk05yE9YklhH45gCtufQcRkll1pRMpw055gFCgCybQTKdwLpXrEQtWUJuclxRzrO45rfT5kfU+evyhTa0slRRJFvYO1HEez/3e+RTvYi0DyLe3ql7yhGyxEq4z3h4kdg0V5p6A0K2g7Rx5/UhFcHCIWRSWecAAelpmRtKl8qr89P0XJTWLRU5w/yAaChmG5eGcZY2zQey3BGoTaCaJhxC/+PfxrPv+ypCv38Q1QtPRLBgEDs//210BMa+YVrpU/T5ULscMlzNoNRHtUqA0fY0rnz4R5gd48jIJqpTZRTzDVQKNREt1CYi4lksoFY1hJu12dT0jOor1U6OTEHqHxegro3v3wo0c4c3lRan/ABsu5ClxZ9tb8/KwzebSqPM6X01MxqjQKEldhI5zDVkM6aCUZSNmhOEDkeqfep1ETJo2VKv0nM4g0hg/VF7mWeT6JMNglQsTyJo6+1BEAuw6IIleOD3t6NQ2Kvszpz3HVVQLRhLr8jt5ufN53JoBlG89MqrsfvRPQgOhjXcKyAWI+8t/r4wxsYPC9hjxC2WCxJ412stkNQhOicJDorkloILMkuQfEJDd0YOpsI1lUk84HhPNc5FKbbp0KSskh1QXFHUDhbbuEqXiTxLFM9B3swSOJmPkZTCBJI76PJovWndI9fnV8bnhpyTK82+uRhbLtXUNQZN9A72IhXN4GB4B172hguxY8dmtBzpQp/BaafnJZxzSL3/2p/auBHSGMMVvOPDP8b+6hCa9NNuX8j+lAbhRTkyJWjo+UsUYnwoHboq4R3fPPTH7vU2rc/3TENAxk2Q583wqiBvVmBpsOtpsYaRhzKRX9azCVQd2VunrzyUjzT2+TVvS6NI7m1IEKDntn/C7L5RTNzwj5g5pgMj734z7r/qnWgTTzo8x31W9J6nyODpJ80sca5mCJF4EqUVwzjz11/FzLZZjG2rojhdQatCTjLmVEBs4NuDYl1IrS3TVqKGxtFmCspNw542U2qe7qxPeRdZs1k5HUYg72SysxpAqIae3m7r04aZ7jRRnM2jUa3pfYylY4boXNyVUh4dnR2OWM8WEAEu1q0G5hABZcRhFGcqVy1NC+Biaklmm998rMslzaRRWob0wRgGTxnC/smD2L3lXsR4T0oF0fz0DIRZmFhE7k9BIMLDqRdcgsl9VcxunEWrGUWjbtkXgSd+D+8Jx2hOTZLOmEalYdI5sqyYqXhnR16bZ+MxSjEFZ9sm7GprRdGgrpqfhndsLdFjir+D2YznePv2ju/zsg7394UKNQKWTCWJzAqoi1prrZgnSYTtS5YxBMmsDWb9X6uVNamwRc6xMayYXbFXnMok0dPXp2wzlIwhtSyEodX92P3cs3P7lHdlPt1RmZ+TnM7fzD4jnL+ZqRLPlRt404duRS3eA3QNIdnVg1DELHk1b5qqrXIVFWpxnTrPPMiNjCRA74mudQFbPV5/amSAiJBQf8IJineWH1IJemDDzWxlOpJmisOer+PB+hPHD13yOb5aTc7RXmCJJHlNRD/yJvS84hxsPfU6zCYaiH36emy89kNoZ/3BZhPbDO4OzHfNI9fYUENu8Dj63/QqLP/oDRj940HMHGihNhMgny+JylatmBsDwThGByMNkAVNdJgLs67emYjqqseddIw31AEDAnpkpm10vHTMFod6oFHjMGeyaU2J54FWzOWRcgQNtUGcn5babBznQXJHMinU2ZBGigxicswgiKWSLmILktTPUiWPVMKQZ1uMRkLhwoln0sj29yGZaUMuMYv+lSPY8OCdKBbH0Qz53nDY+pVCV9kXjqKrqw+9CxdjyYqTsfv2XWiWIqg2WC4YEBONxJUm+tJm755RFIs1AWIqNajGd3Wn6WTtsOZPa+qiy6zI4ZKsjiUH6+NqUbUpD1HyibWhdIBSxGLiDF8CMZVmr5UgV1+fs/LhweOnHaCltptlFWzVmeWrMees9UPChge4uI6Z+VCEQracX/8dnW3ydeYG6h4YQD40gzXnL8Xk7CgK+cIc3/7/tkGP/rf5GSIPi4/+8y+x8XAK9WQPIv1LkcykEAlbf5sBgPpgkZ44MJ3llLMx9k4hyoofyq4ShMyaw99Unpysz+RqSEcEWY2YKsdL/GxhM4Pmmc3hTil9wdtk2oNjjLf+rU9plULzEHCT+PRQww1UXnseFr7rWmw++TpUQhXkPvQa7P7YN9Cey6MrnJS21r/mQBqCBOoXEqKOY/1Nf4vsay/B3sf3ojya4GhTFKermnvKVJAkAfZR9dlbgU1g1xhMmyJYoZdVJGY6Wk0WbJlxma7bXAVlqeMWgozO6GZYMmolPaVYLDdaDSTTUd2PGGvuitVpOvwcOV2gX5MAldH9eAncHOSB9/Z029eUHpqti6w6xVclH7hoKiHH8GKKzjIm3dmOZFc3IskUplqTWH/Zi3HPz25FMxhFHeYVrc3EfrUDClMZaqtDuOBVV+K5329FZDYjsnyrboohEVuoruKCcnYt+/eNoVZpIXC8YJYUHELNtJb9XRJY2BbiRbOG5DPnPeW0Pt4n8pmjHGdDQbyTQpoai5pgI2NISJBg5DYLVqbevF4OaWPrTAIQaZ15z00QQw6zhAt0Z9H9s/6nJ7wwhbbpBWZFxI3MDS4mnzNnZ4eAJ0b/YD8yvR3ItrdjOnQIa89dhmc3bTK85ihgdn5Enb9Jj3z9SHmTL5bxtg//GuVIFxrt3Yhr4yYRallbj59NGAvLDreRVWaaBGpOlRb6Q/a4INwMxHAhsVtjDtwbWI/NHDD8KardzsqFUdgJ23lj2K8VgVxjJU1+NHcRrhnvEWBGT5uT6njGYaD4kuNwzD++BxvOeBsirQam3/NK7PjBr5B+bqeIGElK4o8iYjDZI8OnFo7good/jOnuXow9th+NQ6y/6qiWKJCvKYKZyDqEsbEJRa9MOotcPj/3wLiwGFIqdSpSDBDwNa2RFdiftHTQj4vkwZRxSKoiIiN5g86FIRQqeWRSSU0baDW4cAsiVGh4meprHoYG8vFwjEu5VENXV4csVxhdpL7yWYbIB25iBA3Q6JkrMQhTRANguob65bEc72hDvlnB6kvXY+NtT2K29hRKTdO+MrJwceZzeRNJhBN48aWXYXpvE9UdVQTNxBwrjNnXxMQEUumskUTC5B/PYuzwLGZmiA6b+6OymCjdUdiSMqSejDMePJRCclPQ7jYSbpj3kxsKRyIE570QFGP7i71vWcs6yx4Oqg61YqiRvNHeISdPKqlIE7RgYmUSnxXpq+0d7Sa0JzPKbQCapPMmcrPz655oowO71ZS5O1Vb/LuZEpSwZOlSSnWQ6uhCRz9/bx1d6yJIdWawc9s2M2dwr/nkIGPwuTrd1aN8fja0PYZGqIgf3vIAfnrfNFqJbqB/EVLd/WrFeYop12mZg+LqbJkRvTVWm2+1WXkUIHR/emVAhDTLiMkERpvP0dJc7UtChbXx3UtpGsGKQBFCFDU5CtjPqz/riezzkGRFXg/Pe8E9iRocYbl8GMM//gSeeek7kZ7OI3fNOXh28yZEf/MQkty41CTOO+l4AfT7zQ8P4OX3fg+VYgj7Nk6iORtFpWhuG6V8UXUaWU2cK0qQibYoBw4cUF0Vo4Y0n3N0RAOomkEIuTxTKBNu8/uJ9Eqe6MoA7h9S74g2p2nQzUhCgCkW0UR2kQUoJ1R0toOPQAgb/7EwXS+Y1vMmEtU1twdyFbt7ekVW4Mb21EDWfOLSSs3N1LAJpZxBzTjBXIAuemZ7OpFqzyLd04uZWhHHvXw1Nv12B3YfvgfhjPVVjW5qjDA+i1K+hD+77u147padCNdZY7PGZAlhdZw43rwCN1FgapKSvxomxvOIOg8ylVQsr9wi05S5OMdC5uSzxfvOdg9TwGQyjmicQ62LaO+JINsRR7wjBLb+YwkbyOXBrWqJnOwQ8lNljO8sIKjE0ZHtEoLPZ8MsTx5ebl3E4sYnlxJKHHlnbyNKI0UiVuMqnachBANGMT+nhOOa4ubPtmUR5yjObArJ9iw62zqwv7ATJ1+4FvtG96FW4oxae70Qq0+HrV+rag2xjRpDNWjgmnd+C7nwIKJdi5AYWoBwOmsB0GU0co7kYcyfbzAzkPRBb2dSTPtz6IHscUFc7o5E6szIWoOU1OwmeZ6nnvOfFVDBm2FvQhTZ80WYemiPUq6mVMcTrT04xVPyyER6r93VCcULWzSIgdv/BU9e8T50Pr0XB4fbUb7qRdj7ia+jB3EkXQtANiNKm0KIrT4WZ932PUwcmsL45gaCfBPl2QIKlQC1EoEd1l8t0TW5mJg+8b/9/f3Yv3+/wCC2BKjh9QcNPYRmczZwWYR1Z9BNhNTYYIZa8qWay5P9pQnmQC/WYmHQrpbkCD4QuTbWyygUaPNZ0MZRKhgmAk35Wgr93YP6XUoJo9bP5f3V/ReHmMWujafsaqerZkk6WRrmqSInMb+nC+muNqS6ejFZnMGqy1Zj6x2j2Hv4IbSSs4rMSiFpuCePYfkE4pVvvAEbfrgD0RBrSBJcmMITLDGmGK1x1Gar1zE6SmF5HHkSMlxfWCm02xCGYVgLkJuQBxZ/doajRUJVdPSEcPJpK1FJHha6ykgd1JnCsuZnVmStOLskO5RIl6zWSggV4sjtD9CcjSPCodk6LA2TMRqkyfr4u3mdbKsxS+Kf5UDikHhGZ6EWnK5YKQv152Zgq4n3PNOWVV86mY0h0zOIbNaR/kca6Fnajp2bDagSc3deFjg/w5y/cWkvzOf0wB934rPffhiNRA/ifcuRHBxBjPOZKXap1hR1fe+WtbtIR9q4NvpGskQCoXzuj7avkVmcB0Y09pD/88Zc3MBC4MypkOCTX9BJkbINJZ1Le90i8uGdC1hfcj1Hf1IJn3Xu7GFuhs4khv7wTTz7l19A4vd/RK09jpn3X46n3vFxLAyldcqKG8rFhhbazj8DZ9z8BRx8egwz2zn2gkSHGiqFskgObF2w1tKUPFqQcpaNc+XgZzAksSUHP8q0eFp7WRcjhTX46WVsKhf2CT0QRP6sjdZk7WtqE25GpuIkSgTNKtCsYHziIA6P7UGrSVqj8Y45aEwAl0tvfUrOKMrabu2q1Wgj9Y0T72KMTsyE3Oneagjt5M8kOduoMEOSI6wCJEDZj0gmgUxnP6ZLU1j1yrV47rY9KNXHsO3QHxRJGPHiSeqAC+aK2DaIc/7s1dj0o902uM1EgIhFDeXkM5+cnhJnmKf9nl0HEQRR1fUc68Lv8SojXwpR2ULQJxRuoZDLo9IoAdESzrp0MULxCkplTp8iDdR5kSkS2ybTjB+3YjSF0bVodM81qK1FwB6TW8qY3E2ZZVqZUyxpkxRMKBHRKBJbm6wbmyIwZNNJJ6yvzE1SUKrfqAgk0+cPWujs7taG5AbOdLQj2dmGTCqB8doMjjt7IZ579hmNnqFAgPZItomPjI19XmboWqHEC97+ke9hX6EDQXYAyZ5FSPQPWztP9jQ2zbBJphRH68kS2Ea3KrJz/zmaqOZXsR1kIdhefuMaN9hFUaalHIdAXqy4x4Ta06hpSp27za6O9Tm+P32YJvq2j1hNDlnVUe+yb6J6QTqKkYe/i22fuxn43h1oRAIU3nkp7rvpC1gUTyJFCy1ukgBof+mZOONHn8eWJ/ZgZnMIyHMKm03N0wgWWo06ckc6lTErFkYFprqMUAJ7rN/IBzo9M6u0j0R9LhS5J4gDTEvVrDY9oTZTvxiSy0WnVlmIJQIwPT0htLRWmcGh0e2oVui95LW6jkTChe7wAuPz2n2XKknjWCxapBMJ9HR0YXhgELFIco622Nne7iRm9pQ4lDpUr6LJD9BsoWfBEOIEOtJZlFHGsouPx7Zf7UEQrmDz4TvcLFoqT0Jq+fF6lq04ESPL1uPZn+zQac5+bCQes7k/DsvgY+JG172aLiJoRjE9My0JGg8btnr881YrTBGdhJUois0pLF2TwfAxMc3z5UahAGV2pqCNSnosQTmLKMYFsJ1gA+CYYfH9GX0kDuB8JqWTAcLVAPs2ziJR7UciltIJyufFSMu0XVkUsQoZHJCBZsoqK/NsM7PmJ/PMwDSzE+7o7tThlU6l0N7TrZSZh108nUF8pIH24Qx2bNtCtficc+XcBvKbeN4XeKgWKlW89m/+E610F0Idi9A2tBiRjB3CygxbTdkJMftgYOLn8BvX6lsCwQZe6faQq+zLUAJGXLB82QLz99CRLxh9CdK4ERGs0bRx/ffN5w97JZDoeTbvVfWFK+C5AX1KxHQp2p5G3wPfxN5v/BzVL94ix4vZl6/HQw/ei+HRKYFT5PDGertx0dO3Ye+zh3DgAQ6RLsn9QRPxOHCMzm9y5LNeq6HFjIaOteX+K3MA+hvXaihQuscSAUynTaxsfWabycpFxZRKG52nvqNqEgCxYV4VFArTGJvcjlxuDNFoSbUsDztzEfRAHVHmhA4Wk8+ZWJ7fx9Tf92WZsnGLE7Q5cc16dLZ3akGypJnjG3OiTSyCSiEn21ue0D0jQ4gmE8j29qIYKmHx+Wvx3M93Ip2O49GdP3KsI0r1HJMpaOHMcy5Ftd6OQ/dMqHXDe0ItrMBHaYCr+p1cXASYcrkKWk2OSikgqhLESP1il7l5wXx/orV9I0n0rS6jgSI48jrOrENItKWEPH4YSTWyhemiq+FMRWZtMHlVsf1IYwORNzjIyonvqWEsAwefmUayMoz2bLvUXRp/wllURLSdeICfrVLMI8t+OAUJ1G0X8m58qm1c/wwSqaTKF9a7HD+aaMugb3gQyXQbirEpLFzfh63btiFoENC0XNmDt3PRd97GpQ/yb+7agH+9dRciqXbEB1Yh0z+MkMa2WgYrT2sGQpJeqBSThxZXvG1UlbH+0OFvZTvI/1IPHPmNqwPI1Vi+t0nXRAIc6q85frLjSgoplkcuh/w5SF/hqNFU2id82zevmQp4PW2oiURPL3oe+Bq2f/6HCH3ndpHQ92YD5M9YhsKtv0M2mkAmlMBFj/wE5e5hPPGzLajnaa5dUCQ1T+SQasbZmVn93YvGreHvMwNbENq4nMlKI+1GQ/pgO+VN86g00bHImKKz7ufi1YPhYGMuxXACjWYVk9NPY+GiCvbtGsXE5AxCQVI/y2nsJHZQKKD3axmaHo8yRbQ+qWxjqVt1Nj38rASkGOXVKmsEOH7ZSiweWYQ0hQCKGrZYWKuaTM1cR9p7u0V5pMKkGqth6QUnYNOtO1VH7pq5DQ06BfIwSiScD1OAi175emx+chTl7UzVLavhYiLoM3/zkp9D5PHRVAAAIABJREFUp4tcvozpmYLmB0UTJikUGUGWrNaLrdfLGDwmgcXHN1DWfbU+Kj8r2WNjhw/bHF5NKgirPqbeli/2a/nypQzfmwyzYjGnTcwoqbajyjP6UYeQL06hsD2EcKFPw9nZzlLa67jEnhxRyuc0nEwRu1EXXTKdsdGnxFlY5tS5bqIxOW0wE+jq7UE8k0I004FkNoV0RxI9x0Yx1SphanTP/x5xRROu4/K3/Qtq6aVItfUjGFyJNg6n1oFYM3koe7bMwOTNZg40Kj/dxtWh7sBiZbX3pldwjTk5mZ8DyzEVBjSJ5jh34+tIsX5xUZmb0TNSlKI69UlEnEurYUXgTiT1gVpMK72W11EndVqFm4iuWobBX/4znv2LTwH3PcUGHKZTLTSuvxjPfeZrGEAaS//i1Vj7ib/Dk7dtRTCW0DhGtgE98drX2uS8au4YUVPnhC/k1dXjBKV4itPxr8wp8tU6pmdmdMKSlEEiBvusTBvVxxRbxaKELTQ+3Aha9SriqZ1YsaaKeKgs6h37wKGA9izk+LaQmy0hXwyjVGggN0NeM5HmrJwWuAClG43aOErdC01+sPmxjBocaBbUW1i3fDWWjyxR+nZk0XOBh1Auzmozd/b3ItPdhRBTxUQDx1y43m3cKLaP/xahFIeQtaHWIEhnM3hect4VeO7RA2jujaDJFoizH6J4wlM+2XfloUX/KY7YlKkc6/95jCRiEDxsuB76FkcwuLLGjrMOAx70Skk1k7Y213vl/UxzfKfAIS/xc5xkN8VQ3YNoTBY86hfX6PVF0X1Rm61RrqERaaKVr2F8WxmpSj/SiXYdJH4kjieAsF7kpA4uPTL8GPm5cYlTELASPiFyjQFz6jzEY4hlUkhmOhGKhdHe3YtwZx4DJyzBto1PooEjE+xfqIfLzz86lsd1H/4ZWul+pDv60eo7Fl19vXNBguWD8AWJC1gyEFU2uazfuPwzywWBpAQA78uulJ28UkOnqVV6Ic8hywS0eF2Pljas6sM6cMk0kVxczieJKhcOfXL0LEYTpteqsWWK5rpg82xpIpEWkte+Ah0fuR5bTrsBsckZ2ZYcStTQ9o4r8PSnv4W2/n5c9eB/YirfwrbfjKFUrDvU1lJu/39t4oYhyXxgU5OTc5pbXrCoi06ozfEOpUpF/5eLgxBiM8uWVlOEdZvDyptpaDqtJAJUC3n0DBzE4iWHETTZNqmiPduN2Rxnu9L6xc+9iciZQumO0iCgVongyae24YktE+hsa8dLTlyNZokzm2i6xkyag5pJajBTOKLe0SCMM9Ycj4V9i0w8r/voiKxNa+/0DPQi2dWJVjSO1EAWg2eswDP/tVXSuP2FB5FvHNbnIPGgs7NLm/HMc67Apkf3IThI5NSyFAlF3JgSHrTcdIVCWQdaqVzTxuXfE1kDznjYJZIRTZUbGGlH/6pZBGSOEbRzNjOkKNKOtlgqOWNyox1y7dAi1jIih54T4XXmdj4bJGupq6vXlVvUKhtphob/nH/M2c5BuYXn7plAX2IREsk04gn1H8xtRAcmMDs95TjMpgcmWMcNzWyBXtcCKmNUxaXNtYMlA3vA2XYh1vE0dbMVLH/pWmx9+hm0wjalns4f86eRKKMTs7CFH/33g7j5rr2IJPsQ6xpEZuEKRElEqVudTR67zBVZvzpCkApW9YCspFBP33GWVXrdk12hjWtOFRSJ/x+q3gPMrqu6Hl/39f5m3vTRSBo1ywXZwtjGTVRjU0LiNIwJoYQQev0IBPhB4pAAST4IhCRAICEGG+OAMTYG3LtwwZZlW12W1aWRps+83u7/W2ufM9J/SD5Lo5n37rv3nH32XnvttawuYA3qT1pfixKV5cnqeZpsAfFLBAUCGX70jyAP0y0BWnEBWiJza7jawAcV2g4Uy+Qy6PvJlxA95wzsO/c96NRrKHebmE220HzF2Xj8jofwzs99Hqs+/Pu494YtyNX7MDs7pw+biLnUx2kVMT3Se1OKRKLYRn7n5vMsMNZJfAisfSkOzrqWI3yk+Rlf2EV/vpajPXo2D0+JRm0RgwOzGF9zXAymUqlPXrOdjk1+kDRP1Jd9S35e0tZMo7gpggGnkaq1Lr76P7fLKPwL73kjwghPd05MBRpW57V+/8e/QaXDnzcw7LLz1uOVZ12OgfQqaRTziymjSc+GIm+k+0uIZ3JIjuTQf8F67PjZDkXo/TObUQmPazGTkNKhtWqng0tfcw32PnMCtQP0ljWmE+vpxWpZ78kFz40eCeKYmpxVKsnsl6OQQeKUAiiJGcm+EGs3NrH2jHORTvVgenIOM9PWDuLaq5TLOn0LhTwGBtNohgsoV2cwuzCrYQRpKVMhgzy5bohMIq9WDlUvyN6SxxXLB9jAvjIWyQpZfcxUONpI4sAjMxgsrUSUcEKXabOVaKJHkuBQLUuQ3VRKzKmDLadMljW7lUNMlWXyJVO5KFJ5km8515xGN9LES996AXY+fQiRxFEzaydV8zRzavKyaVVCpdA/ec830UivQyw3gMTYOErLlqPO9daoqw2kCTKK2JGYQvqoJl7dUEVomIuxELl5Q2sx3ptbp0F6r92rGOXsG22HGVDlGSB2ctqN0Hcdw8hrTqmWc/Uv0zqefhKdc8HBc3XjolDyRnYQFNNYvvVGnHx6D+p/9i/oBB3Mtqs4HJRR789joieNq/78/TjzbZfh7m9tRzxizBzJvTruLxehGDzauB0QgeVJQRYUjckYnZleefkWP0RAqp4AKfYrG3WlRwYYtKVswd83MXduFPZ7O4iHc1ix5llE0EQ0QdkTU/zgzK6BUVZfhQTMmm2107woPE+raDqOaBjB577xE8SSSfzNu9+IpCiR5nNDKR3K3PzXzQ/iZNnsTshsu+jMcVx+znqMJS9AKk5dq1Ou6gzHHCLPDfUjwtq6P4mxTedh283b1O88PP8kZhp7RSM0CZ60FEAuedU1OLm/hoW9DDIEEdPiSUsxkzTMas3UBVtdTE/Noc2gU29ogJ7WQZzJjSXjuPT1L8OhF4+jPksYihmWTU3RGZDrSzpRBAqlwUzP4yi6USKolA3i4DiF4aLI9sVR6Ith2fgAqpjHwuKsergMoDZ6xwzOQDrvGJmnxGu9hlatgVwhg+fv3QtMZpDL5Di6b0olmkIyjyDOR3uZGxmQU5FycUGzy9zArMN9y04kf6LfuV75KEXjSTSjLVzy5xfj2YePoTA4gw4WbUjFtW6k5qF6NIqp+Rr+/JM/ALJrECn2Iz++FsXSICo10i0bQpLbbI+xdFFj2IzePFCJjuEztq6szmVPOLgnty5coiJSBcBN4jDdtU3vZ0g4V2cu8s4T04mWmdQIh925tOUMHolqlItvQJ6a+LkEMVwqJL6zHNhMiLozWMTIk9dj5ye+iZ5fP6M0bbZdw57OLCbjHWz86/dhaPnZOOOq83D3N7aj2XQ2iWpSGynd6kPjLbMm40YyTSiL0kJK2bedm1OdSAofa7I6c9MuKZI1JNNpjeNR0VHAgUAvOy1JqjCSxjxWLt+FZHIRrWYUuQFOA+WRTGfUP83mehFNZJBO9yr7Y13IMRi6tFcX64ghjliGtWRELCe2ctKdBTQW66g1FlCj189iGeW5OTzy9Db85I57ZF7Nh3nhmWfhsgsGUWyvwmB0tdH+2Hohw0Ynbg9S/b2Ip3KIDHHjvhTP/OgZtUcOzG5GkJmS1jQRWva42dIbHH05BkqrcODRE5qMKZV6dA/lseRmUHkP58sV1KpNVBumQ3zixKRQ+J6+IkZGR9BpdhGViiUXgpOl5TnRNXcBtZpEYjGt4yRdHUSMoLyNjYAyZaSSf5tjXKxDmzU0W1W9ZrY/iUIpg9JwEYt1utVzGiqJeres0oIpIu1EQ2pDLwZ46vbnMZQeRoQqjqfRD2WiJu451TaJ6prtjQbVSUmNccyx4MYKTRObP5BKskWk0I1OsovL330pnvjVIQyt6CJIT9n6s/PMiSMAnWaI791wF25+YBJBbgSx/mXoXbNGrSt2MiSNxIyGpZqo2wTbDFOSzahcPKxzQ5SZ2YLkkZg2/ya7Zmke11tlcjNQVd3zkvnJhXKx9RM3JQZtZweoKBrQfyhktGVLKYZcYMPm/B0Spjkpw8hlBlDOe1cnfQTtP7gMy771Gex52ftQoNdqq4WZTh1PN6YwE29g0yc/jGUbLsbKS1fhl998TqmkSahyTtY2rPVBjXLJZj5JFFww4lG7vi3THqV+buHyz3wYhOHpm0OgiictR/AUDNhCaNYQTSSNjJEJcfErVmLjRSvQbLOma+PAzqOYmSrbYqi2kE1R7yiKsGISI2wruGdvi4Slgzxnjb8svnA0wCInVeJAIhUjrVW2KDz5Vm8cR74/jlvuuBVbH30c73zrJrTngebBBPoLg0orOxq/o0VKEem+HgSJNFKrchi79GXYcv2zmk+eaD6GVnDSdMUEfzHA0cN3A8654GXY9ZvDGgDoKZEKSjc9Iu3W+uKpu0jt5BA4Mb2ogMfxPhp0jwwPq1TyShNauM4ki382BcdT+timEMLRSJOo1dQPMRCJCLS1WHUSaR6Vvd6YNhb1t6xWZX/TCctziAANRBIN5IeyGH/JEJK9EWQzaWx7bCdmtkxLWYLXRsCS7cLFhXkro2j1kiDLy/qlTFs54pchcpzJ6DPJc8qpXcTjedWstVYL+WVZXPSWS/HgzduxfLwH0b6jStm9bKtknniX2028/69/gD3TRQT5fsRH1mBo9Rqx3yQWWG/pXspbOogiSnIJcxAe2Jovpv2qqZ3QOoeaYzLvZqr8y8IaJnYGOBnp1eRZ+IA9nN4JDWRgFKTjHFUfqFPbpfdMW4oTnF2MDfSojxjtzaEQTSI9U0P6yDzyQQyZ0Oh8nJYRYubSbTbc+3/+VUSWj2HqlZ9Eu07fmTbqQRf3Vo/gZLyOc173Rlz+rvdiYMMI7v72riUShyhyTppVrCanC8XZUpLjBbjJb9a0hfiBiWJyQc7PmbcP6WgLC2XUm019Dr4IEWcutlazo9bJ+o0rcOEr12Pn9p0oT7YR1uyz8D6xnrUpIPZR3KA2g0eap7YRWtjvkxwz+7BqrDMTIbhmmQNH+iIa/TObDNZiXMwiM3YB8owi2QbGNyzD6PIUtu16DJV9DfQ0ep1nr0V61qaF/l40IlEsu3gtCmeuxrM3PC/q4Ynm4+jEp0BCCjdmtVpXxJ+e6cNVV/8+nr99vzIgyu+QX8xgJuRW3NgoFqpVIcknpucwMXEC685YJy0yotAqExRALYAQPPNkeNaf/BmpX4hsQH0rcortz7JpbZtesNZFp6PhD9OHMoUSOfYRXHIqFaT8MSgzh0uojWYHB9dUPbKAtRcMoHdlEQ/+zz0oZcfUZ1YJ1+miTMlcotSSCWIJY4rTTJ954kZiEW1czUDnrBwR6huhxnGAMBrFqgvHsebyjbj/hucwtiqD9OgJE7d3Jy7/w4EI+m9d8bb/RCs9jGh+AMnlZ2B0fBUqi2VNSzUrJA41jeevxUv2FGm6DFIdySJHui1RfMlhR9vLP3UR/CK3WuCU1Afk0yrPQWkKS1ep00a920UlaGO2WUMtao6g6jG5FpDVwaxnzDE9xqFrJz/C18h0I0hH4lgWy6IYSyIZOFUL1obpOMa2/xQnvvsrdL95q8TXNHoWAPdWD+FgtIqRM8/FH//Dl5AYyuOB/96j9IqRh5uL1iCGIFvN42VkZeLklPK5eQhQsX7jKcs2kLxuKhW1fCq1hhBlL1zOh8yNhxTw2qsuw/TCNKYOLjDJVeZgGAAtNHgfTLGQIgIqDQJrpnMhSfxM8q4mvcLvg4GuZSNyGgM0QREbCm93kJdReFe1T1xjbUSYOYETWtssE2LVOT1Ysb4f9/74HqzIjZpCIqCZ6Gwhg0RPH0YuW43U6Bieuv5ZpHIJzGIrgtSihvQjEdaslvJue66B93z0A3jy5h1OEzpts8Ed6kIvuuujvUkTEycn8cKBg1i5YqUc8lhSeN66XxPcnDa4buqNavE6FwquBbLYGJj5/IxH3LTZU4eV6BmmUkpdGWDJ95ZAmsdV2I5r2SY2qVQ+AzMm1ymnLKmJVryG5WeMYt+2HcjHU8jSYocGZa0mUlQa0VohN7uDRq2KTIZa14biExPgNTAQcu1Qj4xkmVQui3YnwDmvX4++1Wvw4I+fx/CqNJKDxxCJkmtl+lpm1cryMYZXX/t9hJkCYoUR5FavR09pQCCdKaOw5SeKn+mVc+M252XIztOWtX/A8kLpLenGxD4I7gYIbi2sNQKGEdzEveTGSQdxVBp1nIw2MUPurWmfIqmFazrKS9QqH2nc3KoYGC4lJkZtNa21g3JNYFVhAL2kqEUjSF16NoZ/+E/YecF7UVqwi+XTboQdPFQ/jF1hGcNr1uOaf/4yOuk0nrzloBucj6lWJW1Pin6sq2NuAH1m1lJXV/96aRJ+wkq1opOWNR75rVTTr1IeRsyVhtQQudHGx1cglyfnloPzMRmDeWCNlpj8ko4SaXpk/lDGhkqGFDjPZMXSkayqZFFtgJs1HE87vo6EzCUI7mw2Q0OOBYRJQTIuphI/n5/AIkKpzglqaIV1XPGnL8Hdt9yJlclRbf54NonSYB/i2SLGXn0m2ukinrphO4r9GXQKL6IRmTUiP/2EZNbVwCN3H8Sn/uFzeOymbSLJcAHnC1nmfTpxzUY1wHylhv0HDyFTKKK/t+TorhD/WYEukXQaWoH0vCxAsGb0AweGigpEdKZfAozcZJml1bwvMZlUe4cBgWP8+SXdaYNdrP3H2VjzI+Z1erBK/K92oB5rM9bC8rF+zJ84jqBu4JQyApVPtJupoZDPaprLanCzRhFTjWoc7CqEXeTTBcxUaMaWxiV/fj7CRAFb7ziEvtUpBPn9CAPTuxaCrtMTuOmOh/Hft02ikyogPbgCpTVnIBZJSGmDa4EIcocEmnaIUqKMT73zYmr4c1uIl0ywkyi2tTg7CIRykx4bR/BTlypbBW99pHYsgulWAye7RBQ7iMaZf5skqRBChzKfcuezgWu/kUm+9kg0R/y0yZkO8KO5k3ptugcr0j1YdtPfIXbeRhy76MMA7SzYL2XWGQUerR3B0+0ZpHoG8Bf//m9IFHvx9O0HNMequpbNcg0RGMVNoEcyKVcCetMI/HLWi0x/+Vl403jaNSnG5cTOadZEA2NTKAReuvFcRWIbAneKjhyyd2OJGtVzXGcJBzBLIXc28JaTMQRqBcXkfMfIzmvU5FWbC8ycFzhL7IcvpGLoSAeLTu+Zi1kpu9LqhkYBqeIhPayQChJlXPGOjXjqV5tR7GaQySbQt2wZYqkcVl25AdVYBntvPwwkO8itnEGQqinCN+pmvcF0+ZYfPo5PfflvsPmGbTqJiEzLoiNus7tSWIwncOjYBKZn57Fs2YgWNFVPSLThBhKRIpdRqqzhCfnzWFamckQePmyFcTCCxAn2N40vzp4xNyazHdmZuhYjf1dOeU6CVTI2ak2ZionNDTEUOxkl9z4aLHAcAa/X3ApaGD9zGXZvfwb9qbTKGvZ3tWkLBQ0MMIMiw4knLj8D8QKtd7WDOFAQQQsxNLvAa95/GbY/fxRzuwMMrouind4nK1jvrMjnVq038fYP/ztmo+uVJqfHxjG4Yo0OPa4JAlKScquW8fl3vQwvG+uIO9Fg6h62lIFxuJ7bivxslQPEyEnw4b/dnFsZ8g9cSBwYrkZDrHvbZYitHdQbzE9NY37vFMon5zF/YgadahOpTgTRkG5trCtNbiTmoHBrHDGNNOULJsWqCEnlokwITYRZR4YBlmUKeN2ztyGaKeLkBR+20SaiZ4yo0QDPYhr3LRxGJJnDO772TQysW4Hf/uQFq6NkMs0hAecWHo8rdSNowt6t6k+mZE7xgBtcZPZWG1XJmjBOVKXcwE1o1Lw2zn3JBs3JaqyRtbEYLWZHYsMFjHiWuhC8oOuA5lCDCGoV61OK8x2Eiqqsr0j14wnPoELAwtd7YpS5YMATRUqHyaRc5zTepRSqo0XE01ejctTI4uxmvSYXt3pzFle+/Xzse2gbcok0hlau4NGLtW96KSqdBHbfcRCNbhXFNQuIpG3OlvIpqhEjcdzw7fvwqX/6NB67cQcyqYxOWzKcpCXVaGB+gQGti207d2F85SrVf2mmyOKoW/+fG3ChPCc9KA1exE1czqfEGoUk6OQ44/LHZb3veMT+AGC5Jj4yyQgajjd5UgUtAotyBDRPJrUc9Xwc0EYJHefP5AXhWOZ5FZZmt4GRtf2YOXEAyRqrQ9P/5qnL0pmBk319BlnOVpMwoqEHBV1rMTYaETTjIV7zwU14/O79qE5EkBo+iVr4InKFJOI06kqYYTlBrGs+9FN0C8sQ61mJwqp1KPYPihE4s7CAVq2CwSzw1Q+8DJn2CbTCONLxAMTAqVbC9hL9mdJZYggkpjBL4MFH87Ikgp8Ux2Xr2YgAx8MOfrZ4FN/83idVGPuWrRCuIDBt5GaI+vQiSqV+qSgsTM2ifGIOE3uOIqg1ETZa6Fa6CMj6cYbYUozgmzrDQyqusiJhsPzAoaeQ7EQxcf77VLtIwJORKBrBi9EKbp99Aa1YAtd88WtY/6rz8MD/7jRjKKKCBDlEljAgnqcAbzYfsCIaTwApVBhVkX+fmplCxGlmsd5imsxTPpVPo8h2Q3YQSal4nNa49yWA09vSInIOBamkqWtI3lSiZcY+4ukraRtOHXWMQM7711PgUD/5uMaE8WN9POW46TUiF1JQ3ZwHJCpXr5tmcYNlwYLb+AHm52dl07nxNWMI52dRjOQxtGI5EMthze9txGwZOHj/CTTDGlLLphGmKCzAUTe7H1y4P/nuw/joVz+BR37wHLLprMTuuIj5fjK5rlYxOTktOfO+npIR+cW+Ms1iZg9ybjxlNKH767+I5PpTV9pU5CzTKlTgH21gqExBNUdrvSnrYEYSjeh05vvwuTVqRH1NsZGDHiLfcPrKPVcOlXgvKNl0KA03l0cFOtbL7TY2vmIcL255Gj3JgvkIxRMS4FP/v9NRz93PQiel1mElEnu99VYMYT7Apr98Be65YReCZgyxZXPYvvMxDA33Yu2atejr71cZdPzkDP74Qz9CmCshXhxFduUqlPoHUG1UsTA7j8FYG9/4wIVIR2fQiUYws9jGkRNtPPfCIew6SKFCUugIUBpDgt2JFf0xrFpWwoYzhxH8b2FlGOuEeDxawS/a0+jEUvj7D1yNs84Y1QcR/Y8JO2+6G5aWiTQb4lT/Y9Rr2Ywsv2RMz0b7QhURDq9X6xqs539bE1Uszs5hbnIarVoXlU4d1z21RQPhBza8G3EaLsWJ3AV6/ZOJDn4+sxfzAbDp7R/BVe+7Gvf8cDuChlERefrZ3GzDjMbI8W22NIvJjXSUw/Ipeseamj0jMvu4JBdwfnZuYUFXTV7uyjUrUSxkEDZ52kQEtFGrin1SBhyCNVJb0KQGbTVa9j3q/AaBshPV2JmMo4+aMZgZejnfYKZ/i/NLUbkupcmOGv5kJ8kLlptdDnu06UxaPRiYFUVNG54tphSqlZp0hDmFM1s7ij+59jIs7JpC34oxBPE81r75fBw7UcPhRybRDpoorJpBM2Kc5obkYUkLTeOOG7fiw1/5OH53024BbMWegtQReR1MVXnSHzh4CIOlQQwMDGj2laCeKW+a9BAXt3yg6EecMraVBTcT5OM94ee0oGHEDKua+Lma+gt7zWqjuNaM/68X92Pq6Gei6w3bmMr2XOeDypVEavi+Xk6HAUW1sPrJZhxebi3g1VdehD1PbhZYyFQ5kTCROZUmEjKI6bkxW/MsQQFFiRwGzhjA+is34K4bdiEVTWLDVSW02mZETtYdA8Tc3Dweefx5fOE/70c30YPk4Cr0rlqHbD6DykIVuWgb33jfBszMTeF719+NPQu9aq12wizaLEVpGs5eD0k/ThPbm7tFKHbAdPq7uWXhb4MKHuLoFf1fIgE2jPfh/33kLeJZsk9IXS8lJBQN4/51Y2Q8+ZQGM/+P2ryrTXU4epYgU1pTcrFTQZFN96a0rchSIkXs9X/xWcQjOew+511IEYlNxkV2JwVsPt7FLdN7MB22sOrS1+Gd//Jp3PPD5xFWYyIPqL4Vq6QriF8mXS7FJLrMyMnWglQWnFUj02VOBFFqhbS+voE+jA70C43W4IAAD6tXKA2zxBJzJ6k3h2ZU5wJhb5btDqZ+THH9VI8GviWMZ20I9ZmdGsPC/KLSSvYbGeGloOioLkojvRgd0XOaPXMYvV4XGGfpvpFeOBNbq1ZQayziirechcb+eYyuWCVdzHV/eD4OHC3jhfuOotibRXr5CTSCOSG4YbuCarmG3r5+/OJHz+GDX/4YnvrJbqSTGfV8+/t7tQhZA56cncKhFw6jVOzVxpV3UoIgVsbKAVd+SPliadzRgpa8kJxgAfWrubl438yDmcGTQw8mSqBa2pVs2szOo9dcDttLhtu+zcTPLyqg0mMius490p2cDBjKxpzDngJMB1iszGGhMY+RoRCxWhcl9q2jduJ6mx1mEjIoo6+U27wMVJVGC2tfsQ6j563GPT/ei77eHoxdyL40Mw5qaidVcbc7EXz2S9/Bnb+bRJAZQmpsLfpXr5a4QHl6Du96wzjuuv1BHCxn0Y2aQAFT4EjUAoyoyQogRiVW1yEeQ8vZzqj99vO3vCn89+eewo7j80rReBrl48D/fu1TeohEUHliGY2R1WsEMTaDCc5EEppEKRX7kMwWjAXDiEqLCykXmJWJ0haCD+VF1Si84fVmFfFOB+e94VrEC33Y8ooPYHCyKlS7oxqpjXoigt/MvIiDYRmRvlH8zU3fxaN37kdnhhs3q7qT18wNzEXGB+4XjG/60+OGpywXDq+BYmDsPVebNSxbtgzFTEapsbxz2GoQsOK4yi6VVapKPqAUEu305P2gYiSV+WUKzjS909aG5EnFfpxqJKVwfsvMAAAgAElEQVTKrI8M9eSC6usr6d+46dRycEPTTN0ZeIiHCGGNxnTikTcrEQMnN0N63uz0jPF/K2VUqwvoWxdivNCLlWPr0GjGsOHai7H3wBwOPjqJUl8BtdwOpPIEQIDjR19AMplFqbcPv7hxBz78T5/Alpt3S962r6+oUUWO2c3Oz2F6fgZ9mX7kZE+yqDqcGQ1TN1E8eZKRZeXacX4+l6k4B+D5JZKFPIGdSbmb9eZn5Hog44nsNAZ31k/MMigqV6FwvVJjk9S1DWwAoszSvIWN3OxscwuHSNsJr00t72DLykh4oAZ1uTaH3qE4Tp7YjfHSiNJ/b5rOZ8uSRbJBZLWlqVNNSZsUFisVXPS2lyNa6MFjtx9E32ABwxvYozdRP1qqRoOkyspL3/ghLGIUieIo0ivWo3/VcnSbLRw7dAzh3CS6kSwiKQZz1sSWLfjxQ3M7sC9t0qXx19O+9+SN/xA+u/sgvvQfN1qNyRQ4AvzL59+PsZF+pAsFFOJ59GRzZq4cJOTnU919GIdvfRCpiRpirQCtiOkwsb4sNQIxbyS33WijFQvQoWp9xB6wTheO/kWjWP21jyJ5yfk4/NX/Ree/7kSE/jsBeZ6U34/hifljeCKYwUK1jU/98LtYrBWw73FaH9KuMo4ux8SoPEH5DzfMwM3Hv1MqlL0dyqUeP35cWkp8XYqDnH/ReZg/OYtChu0Mi+pSqHT1r2aTVSdZFjE3M6eNwpPGo5r8fjLJ09xmWEn898ytdov9R6NecjOSyUWQSX1OCagTOeSMqtV2xTz9hLpakETfuUm0gBIJnezeHlM9c0m+kjwxoxp0anYSzdgMXnXRWiwfWodqLcC5116MFw7NYebZBhKpCCZaD6MRziLoUG2pKetIBtX7f3kIH/rKJ7D5+q1IJTMYGh5AEJBAwpS4hrnZOfQVS0of5QoQYzCxe5FOmqQvN2ahmNMCkwome+y8p3QUiMdxgvO32gQcmrd/Y4uJwZZf1WrD8AgOs0fNq1g9cGk2n6I18Lmq3ylmElvipmjilTL9/LU5Kphel1h97FKwd85yo96U6+B8eRapUh25bheD2Z6l8sXPpMtrKZV0puP2XNkfvuKDV2L7jhkc3VHFslVFFFfPL302ri/yJCqtNl53zXUI08uRLC1HenwdSsOD6MxXsHPLVh0SsVQKMRcUlBI7PTYBul7uibO87A67coT1uqE51FW+6R/Dcq2Nj3/x69i06Qq87hWvxJrly5GqVTBz12/R2XscwZEpxJpdpCi3QhSWi0+9XIs0GrbvGOLpawJC2CJekwni9GHZ/mAkdjsXrW4bfVdegIF/+yxm7n8alQ98E22ieNTNZV4Ti+JAYx6/qh9CtQO89Qt/g/WbXosHfkiyAN+fpxJnNbnIynr4WuBy3DOJU/XhOmactFgpi0zx2t+7HJP7J5Gk8zd5xHSrkw2Iobka5eNwPRFOESVSSCVSJiymuo0zoQlDJWWBZLeTI4/8HUb/VDxp876UanGtEm8JyZ+VxpLukVH95mZmxDUmsslTtJAvGFgjw+cKkjJutv6lpYddCdNxU8zMTmO+OoU3v/4s9OeXoRWmsOGtl2D7zuNoHiZzDJio349uZEFpNgXIZ6Ym0Vfsx7anQ3zkKx/DIz96HoVsAcViFvk8gbEK9u55EaPLxjTN4wVEeL3SOdYEmPlIibXGvr3bbAqCTO2oXhE3v+AKaZMLiwqyslrRYL4NgdBPyRuGcXKKtaz6x+Q+M/X1/V63WW3w3U5gm5F2rbTTZIWZcUpUPWrcaG56Pj9+n6c7sYaZxTm0g2M4a3Q5MtGERu24ljzST2tSormsm0mznCrP4M2f+n384odb0F8cw9gZeXSyRzA5OYnJySnN15JnX2kA//i9R4H0CFL9K5EfPwO53iKObtuBxfl5pDJZxPjaMbo7OuNylRqm3qHzVlguZQad5KvLArXOeAo/f/t/hfmFNo7evwOTjzyDnmpHOsasW+Pqldqu91/EakwEnQLddnr6qQU+XG1cZy/CyMeWiixCNNnvcngLGvLabfVlcdbm76M9V8exqz5F2yGdtCzW20GI2XYdty7sxWzYwblvvApv+ZtP4/4f7bGBfuk/2QynGTTb4uHDZGvIs3EYwVmbd+MhNr35Amx9bCtKyX6zX6Qwmh6ODczzpDaFhLZR5UQggNo+PDG4qZge2khigGTKPVi1vgL1K0ny4O9wMUpkrWvADVM+LjKBTmxZKTW3jVivlDWr2kO+cSajFoiGxqVKccrSlEHSt4p4ijOVnjx5Agu1Gfz+G85BX2EE7SCNDW+5BFuePojudBKpeAwTzQfR7syZ92+jiXa9hhNHT2B+cgU+9o8fxb0/eAY9uQIy2Tj6+3oxMzuFWpmqjD3i+VqWxNPALCK1gLgpnCkVsw1D7g3x5896XjI/L0sE/js3r8Tb2PtlnSy/J1L6rBzj4mdgYGqr9hDnp52ihaW/RkYwn1pj6p1Od9XoJkkuRK3dz3gxRBJYTIaojmarjonpaVTbR9Gfi2Mk14NcIS91EqWstGXp7dW1skzgfHRQiuHyt70Kt3zndxgeGcNseyd+fuf1uPbaa5BMGn2SG/fhJ3bhB3fsR5AdRrJvBXI8cfuK2PrAQ0hn8qIFxxm4nfSP8AExv8wzyXVWrWRz3AdN5y0N1AQIHlp1WZgkYOEGdXkTk2SdRLqId4EW2xrgrKZXdDTNV40guRpQObgWIAegqV/rHP9MCnhJZ0onhtNf9qNK0WQC4w//B7rFAg5d/GEEtRYiBKjULgpQ6TRx59w+7A9rSA8N47M3/w8e+vkBdMuExTrIpvPaELIldBuDCLMhyTz1SGvsoN6u4aLXbMTBgweR7GTRqlcx0DfgVAbsQXHD+tqYf+fD4BfbD+w/q+6MUxzNUE2zrjSyvEYB6ffSqIs5RcoaU0WemN5xQMCDQ1RFPCM6TUmcRgP5bGZpookbeHzlSszNz6NDcoK4z+bB68GgmdkZG/RutzEzexLHThzDa16xEr25AQSJPM7+o4vw9O8OojObRC4dwzR+R9MPMdPKtQoa1TIWZhZw9IUiPvqlj+K+7z+JTCqHwaEeCabv3LsDq8fWIJUxQQKhuKSvpsxFnkGRQUci4uTyOkM4s/uwnrfpGlvQl8xrta6NwI0oUy4OprSYXvJpm9IF00ZmQCwzCGRqXWqEzwKcHywxhpJRHHkP/DXye2rPxR05hKi8K884LskMi1KxxEOIjs9WJ1DvnsBLhlcoaKaiCdXjXNK5QlG6VBymCNoRrL3yLORXDOPuG59D/8AIUkMHUGnPqvPAykrOjc06/vP6B/HYvgCR/DIkB1eiZ+U4svE4tj3xGHLFfs1gRwisatzTmQIwXXakFTk9SkbJdL90ODrZGpvkiyB4bOSCkLmzmQrZEc1tlzDW4lIU5QtJ7cJtUJv4M5sRRUSZe7kBYPVs7YubnI10bmhX3ToFgq7QaS7ske99FomLN+C5V38C2dmKgCARyAhUBQEemj+A59pzIof87a034unHJtE8mUWM9Q0nPNwQv1BhN963JGcTUrWxgqF1vQou8WYcsUQMhVxRtZTUPdyDZxTnBuHn5GmXSZPGZ20HnsBcOPwfr5kbyMQHyCWmf2qIYq6gHrMWdYcSLaS3LeqGciaYwUS9RYeAsg/LB2MuCHZ3fCosAbFuF7lMdqm9UXdzmyZqXlcdTDS2Vq9gfn4ar9y0GrlkEalsEev/6ELcf9cOYD6K5csHMRt5TlRJ8bbpbM/yodXBw/dO4+Of+wgevWkr0tmsfIlypTw2P/woXnLWOTZQTkIGTzFxj01xUKqMGiC36yZQaIi6Dbir1SNPZDt5xc12JwzLCdbTzBjUI03EBdBQmpWL0p/U8qJyLR1OMhmvm5vEXlM4iAsMzIJ4TRL386m8a2fa9BjUGzUKp1F8mTpPLUwjPdBBs3wCq3IjKknYseDPkPvNjIKOgCQcXfiXl+PI4TpeeGoSgyPDSI3slN4VT3c+V5VkzTr+4Tu/xY5JttPHkBhZjaHxlTiwbZumzRKZvKi2HDf0paWBbJY58rqYbfK+MEX3AVL9ZMe00+bVxnUnqMwTnAh1zGECPpIpHQmApEvd/MZUX46ImtIka6X4o15725v8OtaPT1/VdHepTPHj16D3L6/Gts9/F4W7n0eXyvOsYUTyCrG9MY2HascxG9bw0W99DdnhM7HjgSmZaVGs267B6hx+eN+096lvmKhj1dljqJ0gV5XSownzi2kwdbWRRQYWTaqIZ20ax5qPlCg4QRHbSOpZaqInKU4t68eeYo/olLJecWimVQx2Shjrpu5SLlNL5KkwMNinf7f3si//Hj7VXJxbRG9vr4CoQr6oIGR1HeVW6vqsrKXn5iawfl0By0dWIJZM49xrL8evbtmCYtCL/sEcFuO7KBJqI4bMJIjyV6t4+qkG/vBPr8azv96rdlCuJ4XesSzKxznwbm00qmbw3iiu63rtWZMRZpkJkXOr9atUzHQlk2rVGlH0viUQTlM6uieGMHswi5mMSpKWnaDKdCRiYJuXmAC/L0UMJ2jnUWX9V2xdu9c61V0KTZEEn0pzuoeKJJo4Yg8dXTHDphYn0QgP4yVDa5FLc+M6JJktwgQ7FnU0unW86TN/godu24OgkcHAaAnl+GOg7JJlXJZddFpVvO+6X6OaGEaydwXSy9aif2wUzz26Gf39A4ilMzppSSM1BQ4DvtgO4p89ocjfJ9IiPdXWmGGGnAdPLXu5Nq5OR9cz0kZw43Kn6lc7Rf3MrmDqUwerEFWfFnkyOVNE9TCdnIyG6ZneiN1k9R7TreKmjcj/5ycROVHBsT/4AkJasLuJGb7FyXYVt1b2Y7pbwUVv/j38+Ze+hF9/5xmErUByI0yrPEe1WOxR6snWij5kpIWL3nQODj5xDFE6kDurTJlTq/fLn+NpYO0ev1i5wRURXUnAFJjvIzUIjgemMzqdqVRhgZ8zk9YaUW2mE9k+nxHajVRB8gY3Ir9IuvCBj3PK3gyNi8UrU87NzGsUkWljJpMTpdOfSLZgu1goL2B6agIjQ1Gcf94GsZxecu2luPWm32Esvxz5YgTl+A50A+uVtrvUvapJA2pudhg9A8OYeHoGgwMDiOW7mJo9ieH8iGpQa8cwZbU2CVNWzchKLN1ojRokQFSsLvV/GVzabXMSiNiEFH+ezCWjjSY1tOExDwZHsqT4M5TvUYeAmAB72q5V5x3rBcy5AOrTaB0QmtKyUkQIshsEIW1QCDixBtrKMP0mv5oYAi06W00szM1gsvEiBrIJrBkYk2WNTjzO7VIzLR7H0IYhnP36C/Gr729Fqbcf/aM0VntCdS1benJdTGYwNXkC7/z8LxHmRhHvW47U8DgGR0ew9+ktKJJVxdOWjgsJTiNZhsD70GyTi2ClGfeSZwNKtsdbazqXS2WBW0Zfru3nj2058vEGOt1jc9WzNFoTREsypwR1bMSItYw0hAnXMy93spsEUsRNdv0ouRfoxvP/XQ+Q85lDJYze9w2kEgXsuewjoNUwwS+pOyBEA13cuLALk62qdJW/evdtuOfGPYg1yAv2UyVRpV48OUVamFtEtVvDm655FZ7Z/DyyyQwSbLS7E5k3SQU/f96JbJvyhbsXztBMCh1CJCmYVkY2m1MN6GsPDVArG7EbzM0t7eC2qX7wgVYWFxS1uWFtEZtIGiO737iq37xxmrtGKlTy/fj6DAILi1Wl3BxlPAWQUctpUdTHZHoeF23YgG4kjvPfuQn3/HwHBhJ9SOYC1DI7EEQoisfAydqwpfo5VTgXEweraB/rCkAZ3zCKY7snZNZlz6qjU4drgggwA5ykZyjy5nji0jB2QxzS+2Lv2g0fcMSEr8O61Zip1ttmj8bqO9akBgoKdCJgSe4320cJ07TW4LjqbFNT4cv4UT/7Hadppjcw6SANqstnmA4JnB5qOjM3Xrcx1BjcqTDZqDYwsXAUtfpRnLtmDfIpuiPwVEyimMuJQHTRuzYhjKVx1w1bsWzlOIL8EYTJSUQidr3iTXfaqHUDvOPTP0OQG0V0YBWKo+OIxUPMHJlAtm9AnRKbCIuKjimchLRWlWI2fMLRWj9wov3oWGgCsPT5Q9u4OgUdxO6lXsTY0H0I0abDPJFibl9fx0qmxrjBegAauHYCc6KuWWSkNaSLDEsnNL+/1CDniVssYPj2L6PS3499V30GqUqVk6+ajOjwwXY7uG1+L17sVNCMRPD3v7wJB7eHWDjYRk0Cb4YOU+jLZESZZDfwmj96FZ5/8lnkUgVNuzC4MLDwRlMwTSi0Nok9SC4e2o1ysRoZg4CKtSxIOuDgtcUt6znqlHdTLp7mp15mtQYuWHF9azWUeou6LvNqtTaG94IxQTbz1zVAoiPbDn5fPWNJqhiyXK/ZCKM15SOYm5s1KZhqBXPzM0gXFnHROeeh1uri5X/1Wtxx/e+wvGc50sUoKqltQMC+qaWq/Awc6B5ddwmeu/8wEtU8xjcOi0dbjPcYi8xbmDoqIe8zUXXSGvllFi0R3SNeL+WKfHvLVD5Dsxh13GbrRds9NwsWnqyUJDWgy6fdIrQwhXTaX+rLcrTSrRsCWkJYnTqkP5F4Xww45FqgTWdCyhFiWAmLYW+ZiLQJA+rnKB7XbGChXMbxyd1Yt6KEUjov76BcOidKJLOnTR+8Ant3nMSR58soUGu57wDaUng0NVQBYN0Odh+exRf+7QEE+VVIja5DaflqzE8fRqvaRLK3T9x5dll4/WQJ+iBH4pP65Kdlrr7T4Q9WtsqUHfP/nhq6QN5BYn84Lx+lYFKlt5tHaqLsIW0f6xdtusMI/qK2ufpORTSTNd93cv64Ek/jQ1JUMSKXAAYytXqyCN5xBXIf/DPsfc9XUdx2GKGrMcmkYozZPHsAT3RnpSzwse/+C7qFVdj36DxadfJjCSjZbCW/WLtcfNV52LF1J0ppRx7QWCEDvfWa2QKyFMsQZY+amqAYh7TrOiWLhaJtNvn/2KnK00AGWg0j2osUQMnXuBFBuCEqi1W1pPjgyfbhIjVE0NXMsjqpqHfL7wlkIpHekTG42LgZ/ICBwJ66aSHz9/h9gl8kQ1TrLczNTyGZncJF55yPVL6Is992Ee67/jkMl4aRzHTRzO9Bs0WXObsGRvf52VksO3MTnr3jKMbPXIG+oTwWDswikcqphSTwx1ExfW+T/GTW1MwseLKxx8375a1rFNYc51jZBck61YrWjW1cG7D3X6o36zZIUOrrXQpexAHIIdYGVWpLsoXJmfrSTkir62Dw2fN+SczeqbcYW40kDL+5DCBV8NagekcbmVRcDrdPTB7DzPx2XHDG2eZkkM4hmc0iSAa4/L2vxYO3bUdnIY7ScB/i/XvQCo07zo3rg/h/3nAXHtnZRrJnLaJDKzGy9gzs2vI4Sn0DiBd7FdxYz6ssEOEkpj5zwDlhmejBJta4R5bISjbUwnvpeRLBs6MXS3PK+wL5h8WXMHBF4PFSrcdvmK6ytoHzZ/HppRG0pUFMdUd56FqqpBNWEx2urcSGrUuXooko4meMYeDGr+DQz+9D4ut3oJUIbIiBvOVOB3vrM7i9ekA3+8Lfex2u/tsv4tH/3S+QhuR/EgsicdMzHjt7EEi2ML+/hnQuiUTEGFGGk9tMsdExzUTZQ+/sH9oYmRHjGQykc+TYTdrwrs3AB6bo6NJkntr8nAQ7uJDJhBK7hxGeSn6uByn5W6dgz3tNEoI3txapg7alAmH48MwHlq9LCmCrzkDH8bgWFhgcSPbnMECljoXyLMLISVx27gYUV4xi3ZvPxYPXb0OpNIBkpoV6ajc6odHzOBjBz0qlzNVnvxI//taD+PQ/vxeP/fQpFLI9qv3ls+PS/6UA59M0qydO8YOd+L0tNmOK8TPa6Wajn7z3XKD2/Lk2DMziZzMlDVsjptNt5RWvT1iHq/kM1OrqdbSAtTh58jeEa7B0s3LNnrMnZ3AjLAGObhSQPyHMgddIZYw2Qb46dh17DGsGSljZN4I412U8jdKaEi6+9hX45fe3Ih6hYF0PUNqNbruu4Rpz0ON67uJjf38zjpSTiBVWITG6BqvOWItdW55BaXgUAZlj5D+TlEIEmZvVMdKoeWYgccRQf5YFEac9zcNL/043DGJGAYKtIy8/JRbnTkneoBhrU4cE+5NCD1CkDIuYlmqae7g2tJN1JaTO2VprfViPkzef56wHVlg42AO1Af1EXwH9d/8rYtUu9r/hsyJ3sNdFyUve3JNhHbfM7kaVs4p9efzDnXfgwR/uQyZOXWVyUFvSpx1Y04uB0T6UJ+jDQqmUMvpKTP0c2OSmLeQzG7MmPReMQCWJiiVMnFojfM7KwguZuRPaVB1MTpWDF9x81BAyj1x7KP4UlxCBQ1k96YLXKxYPJYGc5QZrMVIifbrnF52eBetxPtBGS71QlgIsU7jJJyYmQLdDMoGmZvfglReci8L4CFZdcQ6e/PmLSNIwLdtGK/8iELAt09CDF4BDe8vsejzyqx141yf+EIc2T6gVR0BJ7BwnfSt0XsMbVOPIngZOmVay6XrZXK5lJ1zEhj1QRJ1fKgeEbVjqyr1FUIe/w03ja2Kesja/a6kjnw0BJVtHlk57tVCmzEKl5QYRA0XTddqTwdRsCzzk/WdQNVzFVFGMJmm5BK9loWxgGjf/8YXDSKcmsKa4BslsHKl4GmsvW491l2/EL777FDLZHEbGc6im9iDomqyqyeoyECziff/vFiyiB/He1YgNr5SiSKNcQaanF4l8QTRfL+fLtNnPWBN38Iw9May5lxzeYofOqUCnTb997NLQI1hEkj2rxxMqfCrp20I+yWFEYP/Nn2AOebBI1zUtYf2buzn8M8EQf9RbAmyRkUyeZUNDKP73p9A5ay12XPIh9FIbi0U8a0m2Gbot3HJyO04kO2iGdVx35x3Y8tAMwlmDzaS4H1vExks3YOaFGW0ioqZ8h9mZOZHmrTfm1SttzMu3I5jSSjZGd8gWmAm5mXyNMgbWbY5AwpuptFgqDVTEJ7BlWQi/eLIYD5kLlUHBojK9l7hYRNhfLKNUooyrnTys93p6Tuk6GzvLakL+TmWBKbLZiPhajekjpT752oeOPIerLtuIgTNXYPDiM/H4z3Yimy0gmW6gUzygul896oap53O079jJDI7snsc7Png1jj1xEulE2gUfA4P4VXWeQAwUlm055wtHDmDQ4joxYNBOTKs7Wb9aNqa6XrO1liG1HEXW+MWnnChIwOCz86eu3/Q8xetSyLDX8/8u7W6Bgk0paSylx9y8TlGS18UAGYtSY8oZRPOaXI3M+tK7O87MzePw7G9x9tBq9PYwkMbwpvf+HubbIZ781SH0DBWR7VtELXEMQViXtKwtGTLaGnj3Z3+GTqIfmcEzkBpbjemTxyTQx42bLPTYmJ6mfeLamL43K4MMch1cGaOSSlrShgdImCAwfWUNmm4feXl4qgi2qGSwtJvGcI1fqyu4QSxD0Wnj+r4Wu2yEzVpJdkrwxrHuM3DAjntLdwzU8GNUZGkN5IqIXv1ypD77V3juqk9gYLYhoriiI1sp3TYemD+AbcECupEQH/vRf6CDFTi0mT24kKIPeOklG/Di9gNIMd0KIwpCSkXCrto+kuVUe6PtLCdYn51Sm2AarDE0pb8eLLJUyNfmekpMs2ocjK8jX+BgudrmOn0NYQzQdhGfC4r3lAuaG5lUQ6tPTdJUJ4joeSbnygejf6OKQpVStTZULgvGtg3b8/e5IaSEz5Oi3cRiuY6F1hQuPWcIoy9Zhb7z1+PBm55BqYeDIh20Mnul9MCNR++g2mIFYTSFp5+aR7cM/NVn340dv9wlIkgu16P+NEE5kd4J7DEIOuKCyY8aCczKB/PbVe1GkobQ0oQGJnhSW2sLyOcKCmJ+Tla0x2x2qe+qk9hZ3XCteBMyOw1t8ovvytdMJ1Ogq55mmsnQ4sL3eINM2hg0TJOYJ7G3pzz9JNe6dVkin5ECcbWGQyc4mzyPlcOj4pxf/fE/wjNPHcXUoSb6B/oRG3oRYZScddbTxuASyFWp4z1fvBVBuojU0FmIJtNoR0IkMr3I9BQRTWfVnvHlmW1BZnYxE6B3Na31cO3z0J/JU3gpV2RYTATB7uWX+oPP0juS8qWImHNop+kpaac7cEWuB/Jk9U71tnT5u+rziQHiCnZaUbqJGp+WKgR4UEi1TQulbB4Lg1mM3fFvOPqVH6N962bz/KHyA8fx2i1sb81gc3NC0z1v/9cvYtXZr8JTP9uNdG8O6zesxuG9R3RTmIYnY0nN2JpfkW0QpkJyqKcJssbkLKAs8V4dWd1HdC4kXic3I3/HpFMa0olmmqcb7ni7ipCyhHSDCm5I3BQdrNerqB9ACLWsP93pLlTcUdx4GlEgTf1TaguTsU7pVf5OpS7wRWkfn4mUIpjutTA5PY9KdwEbz85j/CVrUdpwBn57yzbRGAv9ATrZF0z+1WlwVRfLCCNpPPrQBAYjWfzF378HT962HYl2QmqDYtPBTMD0rH0dq7TwNGacJqtaUr3wih0e+VTG0ek4i1XTRPZZhA+ACvSOJWSKkdbz5QnDTMfzc8mqUkakn3X2ma6OVr+eo6ZsIaq9ZKi9rlsaxca29wFTAcBlVabfXHNGajT/aqNaKWP/0d/h7BXLtH7e+sV34J5btiMV6UWxlEe3j8bW1F2O65mS+cZW4ez0At77d79AkMoimh1BrVHD0Mq1CHL9SHL6i1hL0vAWyxhs4yqbFe/aqJ3iO2jzdtGVbI2RMyRpIWvbLoLdY5cuORn4Rrnl7ZYGKyWkgqH3u3WbTm+oOsZACD4AzTA6cXR/QT5NUprqWiEmoO5qHd5URaEIYqU8Vt77bcw8sBUL190g7VsnbSTPmqPtMn5T2Y9y0MAbP/8hXHTlH+PuG7biyqs2Yd+Oo4iFEGXN4Hb2vCgVyjYCwR5OACUNBVwTb3QAACAASURBVBZTxdIbayNxkTjK2WnUQxMbM7IIPyNBEYmOU2vKjZx5fWhFezkeGEBC4gnvp05HTcLUMDg46OZ5rffosQJmAn7OV/e7YsLs2iDRmJ2ynHBp2YCBmDSRuGprkvZJAaSlRbnTwDkX5TA2MorSmWvwwM1bMTI0hHiuhjB3wG1cowmWFxYQRpJ46MHjOCM1inM2rcUZl16EF+7ag3KVxmj0ETIFCGPu0GjMaXA5Wqef3OF9phm2v07dM4chMHiaLA3rSjs9fGlgizO0ckjgyylfKqt5rT/MZ8ef4wZRf5ZC7sQiWM5wnJJ9Y4KhyugMe/FglzGv7NDxPV8/oWROF6HOH95v/l0Cdd0AR6cOIhudwdr1q3HFe9+Au36yE+lEHoWBJBKDvJfMTo3h5dtRB4+dxMe/fCei6TTiCTouVDEyfi6ifSMIqJsdT0i3mffJNqsRaLS33OGydDg60wD1fV1m1glNxlbFyu6xy2Wz6dnvYgG5WGARsKPepi0kk8Rc2pRehoQbXBMc5tInbWZPtnDRWUgjZTzZ4nBK9fwzazOeIkTQSvkChh7/Dqo7j2L2A9+0XJ7TKIyW7Q5muw3cVjuAxW4LL33HlXjt296HwexyPP6bXcgQhEmZUJdno4gho+a81Q6iw7m6kbWrXvi0TIJPXOkfb5T7XZIguEDYtuFDVt+NKQvTadce0qLUInR1BFt6ra5TyDCghikh081Oq24kFeatdFuv17UI1cAX5c9SS2YHZIEpqGh6hsCSSZuK/OECDBdQo9bA/OIC5soLuOLtG5GLhYiWhvDQT7diZNkoIqmT6KYOgw9eny/oyn40CJJ45rlpjAcrkUkmcOk1mxBms3jx1xOoo4pItItEGENIdQZZUHYQ7TozNUdL1MZjuuwGMvQZ2i2d1Nqg/kQ5je2kZ+ACuQKRo/rZgeG7ECxvjEHlBc2ZLtsYnAn4i4rqxAmWxvHcbDXXH19bBA43G670O8ZAaJJA3PAyg2sYgYanJw8RBt7JqWk8u+VuXPO+N+NlV7wcD/3sRbHC+saSqESft1ljR6Tgg2SgOnhsGp/8+p2IxTOI0Y4iFkHvygsR7+1Hh7PeZJLRtJxZmKWd+nzClVygs31oJ7F2JX/PeVOxzcl1J/R+z/JNp/IehxT7COVTItZporsJ6fPo8almsaKc4wsL0nZv6us3f4PVMA/ow5IU/Ywb2G5uG41uB8v7B1H4zT+hOVPD8WuvWxq3s/QOmGvV8IvafsxHWlh79cV4+0f/HlsfPILeZC+iEfbHDAkXgun6tdLn9Wn5Eo/YWhbyQfVyK6fxcDWvyeEAmkUXC0Zsd+LmYgZpUsoCgp/g8Owp3h+ioNXFiphRsiBh+8MRDKhW71Nj3ikuLO5BSqVaimj1Ne+3MaYog2qRWSqJAjSkD+vaSkTTG3rwi9VFnPfmcWRyUcxMtbHv8RMoDZQQpI6jGewz+F5JGXv0BDwCHDpYRW9lVMBNN9HBS990HgrLVmD3nftQmaUaYwJBzJU/zLAoYObKAx+whNTyfy7NzWSy+oy8h3SC8Pffja1YUD+dyHPa9JEvT5ip0AicbTCF09N+3nAS27Qee+Az47NgENSn5HpUIHTDIW6V83eNd22ZlhFvDPlWQHTWNvze0SOHMHxOGhe87gI8eOMOFHvyyA9XUYnss9aNzMpPHWS79h3DF75zP0BdKOIRuRzSw+chmu9FLEcNK27cuJzo6VniuQMKVk7myPxxA6XiKpe6xlPQHtAZbZs02Ltik1JlS1+WNrr+7ml9HjRQu8RB9aYaYVQvnzb7B8oTwvpN1nc6PV3236N8DE9Gr1xB1Hi4p4TBn34JtVQKU396HQLnym01UxQLrTpuLb+AmWQHF7/3arzkgj9A7UhWxHBq/LKSsVSsi2w2s+Rw5pFkf6O4WQmc8Ob4z6h0x/VVGY2LPTxhnU6wd2Vwo2QUaGMqafPHlkZazQTnWdRFf4lD8fYeZOH4E4DyJYywBvQYuYDXayoQnSWKHj+Hpm3o+sBUVSvXUmV+JZKkQrpB8m6AVDaDcrWMNVeNIozWcHxXGQefPYGh0UGEycPoRg6Ic8yNG+XIZtxE7SrTDVSOlBCPZZCkbUw2i9zqJM561UaUJ5vYvfkFBLWkVBl4DU2q7bsMw0zHHNWz01TdLz8mV9fq+p1mlB9/VOotewNPBNE2toXp5I7swCBK7Vp47nek6OgIPD4dt/64pY+MSQQM1cryPyuk36RX/X23zLGzJAdE8I3BVm1Luhh4NhuDcHYCG1+zEfddvwOFQgaF5VMod4/rkjWwIA65qaLs2HUU1/33g269A6WBMcQH1iOe70OHBtmprH6Hp2087daAH+tzhgOWevvDkWm8gZW6fxF/KAUIdoxcIuaUb9N4YMZQ5FPyofqg3KRuQkhC4K5G8RtXN9ydCL6INgc964fyQ/ovgjq8UaoJw1Ath95SCX3f/gSCdatw6PWfQqJtg/F6qEGA2UYZdy7sx/FUA+/73jcwfzyHZKtHahFcxAQZ1Bvk7zj4W5HX1ee8Po/kMoAwHVUEdEZT3pKT12u1sVHiuDgZufV9iZbbtBDracmKhAQ+TDyOBHUDUMzvxdIxN2rlepCkDfL7cQq7OxE73gu2pHif/KSJ+qcUQFetHrd5VV13c0kAT2qN7GV3A9TbC3jZn23Ai3v2oXqiiYkd82KlxQv7EUanjLhAxDcWaEiC6d7ciSlM76Xsar/xp1NZoy4mA/Ss6sP4xmUaQ6vXotj71CFUjs8h3o4DHZ6yvCd8RubiTqoFRQAJDPr6mOORzA70HGCnndYDw6ysVt2mk8gawSwG3axlE8qcLEngNYl+q6EGYytJh15kC1fDKkMhU6umZ677tZRJOdE5x5MXJuH48nwdM9kOsFit6NSWiigNrocyGDozhvv/bxcGh5ch0ks3yZrxn0m66YZuVrqNJ57Zj2/c9Fs0W1QETSJJadaBM5EoDSOeTCGayiKgeXgyBRYtTIE9wYbrm2uB18z+tIIz1w4F4pzwvxqSrssS7FnOGveUIJXfuKf/ly/CByFUWObXRqZYSkmcRrD6jS414c3kw6JQuPp6px/nLsbyPZQSqY61xTn89Q8iuPRlOPSGTyPXcmOCtO9otzCPJu6c34/Fnjiuu/NWbL5jL9JBj5QCeSOVUrgeIk2lWYP495WcqNNdVr2rVMren5uQ+lS+Ac5/07ifs+10B4K1Kpwxt5HuKXQW00A235ug1RKoFNhp7TeiT8WkHsJ6qlrR0IOXOl0qRVyNaKdGIIEzWb6I9GLfU3bkUkeiokRUCfxU81Vc/ofnY+fWgyjPVjC9awGZQgrJ3n0IIxxMMPUInrj5Ql4LfG5qAhM7ExjsWa9NyAkXm0VmfzSObjxALBVBcVUay8Z7kRjoRTpGzKOL6gJQmamgXWmhVWmjQqvQch1RyuxSmYQ92UxS/GaVMV0GNNNCZl0rE2s6CHAZkxK5pPllLTC/vvg81CEQJ4A1vu+XG+XWgoIBTHxG9P7VkL7zHGJ/l7PAqqdVG1Nvm1NLTlCO+obuvdXB4KQPSxwy/XozOOOSHvzmxi1YPj6Cbv556VJbu8okYw0TCbHrxZO47tu/QbPTFc85nutBduBshNmSAKsY0WZiAWSmxVNyP/AYAWEufg5+ziWlGAES1t9VOeJKFB1Ep29cf8r6k3aJLOFOTZNYNZ4rbxiNlJiqqLZxTCtLfE7l3F7027+mpQJ2CsoYiZQzUgMYvQCs+fjbkH7/n+C3V30UK8qGVMvXp93GRFjFXdVDaPQk8LXN92Pzz3ehlB50DB1rm0jIu1wG9YJ8veOjrrSgXL1gLQMzxubm42fSxpbVg33JOtJ5lRrybKm/r1dVL8m825zn/eSKofM8BZymFJlEro9NYopNv3A4gGbOXMhOtYH9YpeeG2pJdNrECHTiO/oogyhPNqZ3XOy9Pb1YqJWx8ZpzsfPp7Yi0E5hemMf0zjn09GcR79kDRMwzSUG03VJmwqBVWZzG/JE2wuoKFHIEw0iJTKAVcMwDSvOppdWlFZVLtSutefSvGEJxKIV8Xx7pfBbRHO9fwnSOSRqIJBSYEMRRW2hgenIetekayuWGetxBlfeS12IBlKNs3FynCRwqoPN/3IBMmy2F5J38/7P6bE0ZCGUDDKauweOWfV6eYr525ikrySKHJ9izshaNmXzYc+e9oa1KkIxi7aYSbvv+Zqw9p4ROcr+456daVoZL8HV27T+Ov/v2r9FodVHK9yCWzCPRuxpBth8R6pOls4hQNlifk9pqrsxkXe2YZsoKXWnFZ0X7Hz+UQIM67jdNtu1adlloub8tSH9TGA2NIma9MN0uQdTWC1SN4WoypsAk59uiMzqg0jn1Ak+dEl4ZQYigkzXh7zTCNuokm7ebGLzwbIze+GXsuu56pO/5HbKIo4Y2Yh3gueYUfls/jp1hFTc8cj8mJ7uoH+CiJwOqjXzBxL2Y8vLh+S99BqeeR+6sCOzJhNQdlEW0O0IUJZXqanuri63u0kkrzV87qWXYRITcyXiyhcAHL860U4VU0POMKC48ybSaayBTdD4UTkWRgC+dJFfHGVhCAIs6TbWlsUiJqUmPyaReI0EcKVJOM3GErS6CVUmc+fIVeOLmbSiN92KhXsb+LQcxPDIK5J7EYnlOWsFMfPK5rDYJwaN6dR7tSgUTe+LoyQ0hESfRnzO7fPYkgiRtskbsMT5jprRc9xyuoMMhrVhsjI/3Rsg50WvNvtaRHo6iry+P4dF+JEdz3McSGuc2iVLHmeJGHa6TuPrU88cWcfIwjb5NkysRMIvhZ66ArhEm4UJDL6bCMcQ6PHVN75ubnjRVM++y9cr/cdZXgoZKnwlW8tQzQUGfkUnFhYGCZQm1lN3maQYNnP+Gs/DzH9yP5WvaaOOkNg/XNv/LLEvYSLWKk9OL+OCXb0Y0bKGY60cYTSJfGkMrKCJSKCHd04c2a13SOpPmwct619x0A/XOI27dKlsjRTgw+1hPA1VZ6lFlY07ZLK1P7yzyGnOJNYvnzmo40X2JrNF2ekhNytMw728q6nok9RTwZULPnm3jidR8DTrz8QM02EboyWHNfd9GcLyCfW/5HNJBTJukFQnxeOUYtrSn8UR3AX/x0Q/gvR/7azx77wtIVFKYq82ikKd9hkVcooJ8L30212wn15csGm5Y3ghGVd83830/RTmv8+NaHYymBCwYjNQPTtKGkekigTDrQYvwH7OUlgHPExf483QmYG47MTGpxc9eMOs4WXW6WtvkbjquF26iawoiAv8MOCTvV7hAIq4WXZXDC+0Welf1Y9Ur+vHsXS8g1kgikgWG1w7hvv97BP3DGSy0NqO3VNQzpCwLhc15zby28sIcuvUqKrNNLB7LIZPqRyRISXybJ6icnzhS5wYA+JyqlbptaJU/VMCgxI+lpmq9OcDKwDtiGDzpjW5AlFQTWgku1FCDIaneqFT+ewd60bOsoPtLjCKR5eB+KCPz+myIykwV5dkqZidm0W0Q/DSZ1zgoHMishOyziAzCtZ516pLRRz9gBlujD+oEk3KFUU3ZA1I7jrPCGnInRx4IYyHWvXwEyVwCv7zxYYyuqiAar+nAUvD0znyO8joztYh3f+ZbiKX7rL4mFyKWQ7JnJbrJAuLZAiKZNBLpHCIJU9mQwoWE+LtC4Bk0/PS7AN6E9bo9wKqSgJnToXWvC/2mtDrWC3QZUmrtnVMCzR4GFxTvQAFLv6y/JFKDyDCWzrB48b1TkhL0ZwlVGxeYIA0F6ViTVlmUR9rYcNM/o7VuFfa/5qPItQKxk7qxCO6fexG7oxVsCWtYfebZ+Nev/TsGz16LrffsQWe6g1jKUGJDeS0rsGsw5zfOufaV+k0e1G1mX8uLtkeXP9eK8emw/7zkFfNFOdhuQe5Uz5GR3TjAHCs0CiPfn5tX4Iy8ZiuiKdoQvtExfSrD96BAnI3HiVi6BOiJI622Bnu7bTGomMqSUdWNtHHGprXIroxg29070C1nEUsZCj20oYSHf/Y0cv0ziGWO61kxmPb09iKbzmjRzM7OmIl1bRELs9PolNtYPFFEMtqLbpAAurzOtE5go23SGI6v46RiHFAiJ8S2pbFKIU+b42UdZ+uLt8aGyPVcQDqsDYiE7BU71h6d51lmtMIGFluLKPZmMDw2gFRfCsX+IlL5JHJFyr8YZhHpRNCqAfOTZSzMlrG4WAWn7VqLvG/UvzJ1RD6QWo3WKXQ/NOcLtdt4vXSld2L46VwG0STQP9aH1ecNqwW3/cnDmDo5gdzAIR1ZrMoFIjmwVevfWZ1UG8DXvns7Xji6oEDRDRNID64BkgVE4hlEklnJ10Sp501AjJkWNyuzJ1JGZcPqZsV5rQQAHWnII/PKfk9s+P1Q5G9q87imtk4hl+Kq1nNpkicJeLjeCn3H63UHsf7ON3cMXl9fGrvE+KMaIXQSI0JOUVedSznWWrOF9de8HvnPvxc7r/0ickendaM4QHXf9D4NGdzTnkY0XcQ3PvY1jJ03hjWXnoVaO4bdjxxApBJHrEVU2VQVuJGpjMHTdXhoSKemUn1GOIdYE5klt5arq1JbVBptTCjr9Zlqvnn8iEXlfl8b1IEjmgoSPbKNSr0mLi1V/0I29Li4iJYWcmhUjV/MhyCvXFdfM/DZAo8gQo2neErvX+8wXSaS3EKWCov0xmnX0bd2GGsuLCFsdfD4T/c4+46I5GKDWBK5lUls/uUWjK2bA2LzOvXUVuDMaqVGvwCEHTuhpLjI0qfeQKOyiJ/8cgv+ZNOfIuykEYTkc9sAQUvSvIZxcNNVax41tyF1lgE8pSnnw40u2mHcZkltOsurXri5Zke24L3RhtCpbkP6BNx860snE0dFHQrMcoRrqFybRyIXYmT1AMbWjaBvpBfJBIfFI8JiVK86HTLZhEgVzEAv9r0F+vAanK+xDioYxbbdaOD5hw8gbMZkU3L05GGkSy+awFMkoplkG4K3TIIBlfz4Q4eO4Hs334VnDtQZwsUviCRLyJQG0QwyOmkTGQ5+5MWkYk+XG5Y6VAK5JMrIAKmIgxgzFr4SueKntUeDF9ddGeYyabUdZGTlFiWPa388nw4w+UFsq+GMZaTC34EB4ipTv8lNZ3he8hIBwZ2EJlRudXEzbFgPNuyiGQ0RGy7i7Nv+Dfu+/n9I3/GkHlol0sEDs/txMt7Br7uzaIQB/v1jX0dvzxC6yS4GVpew4iXjiGRJK4sDrSjCJk8HXorxO1WzO41nMbJ8K2JphNF1FEXP7qJdZ5pm6gmcYZWSvJArO8m9eBdBllq1jaBMd/MG5mcW6djp2kldDUb3FovKNDrOJoW9Py4Cj4h2OObogBciz/Qt6ka6ohISACr055HuzyKVjyDIdNCttrBt8x5M7KtiqKdfgYenMp9LMhtDelkCd//sAZz9stC0puQcaCVEX28vjh4+gBgBNPka2wLn14kjB/GVb92iAY8zlq3HZedfiuH+lRrcCEO2sKz25yYNWKN1CM5YSs+U2tzzbCZW7cMo2WZ+3paoadK1x4zAYJ2KU3JBasdKrMCsX4mae0cIBVN3UAiLWQI5+WfTV2q362h36+hwTakHamm3viJsxcSRpH1KlHW4PSNtPjG5KDnEv0dRyPShHdBDKI1Sfxbl9hGE8UOmONKwA4G1NF//FJ7BPv4ifnTrA7h/60nbuNEUooksOpEU4mwPpfOIJXNANI0wFkUik9WwPliOsDxJmCg781kebrId4FbzksgOXwr2jb8mZORh9OBp5E9IRk6fTnLj+pTR+LvuPjjqmT74aRxlGfY6Rgk9hITeOoTWvE5PQdsCHtp127QUCIuFmE408erHbkJ11xFMfvBfEWu2cDLWxmOLRzCR6OD29oxO6He96R14xXmvRiKSQSxIKlK2Ig0E8QCZXFILvo0W4im7uUbnNObREmLOWiYamjGx5nEtbbHxPa/9w5TqlEoGvWH4JURaEzG8f2l0YvTR5YJzkx3qJSt51vuKJ+3IzUorHbXN0HzdeaGd5plGlhlXVhP1Kqd/aqhNLWBxsoGTB+YR6SaRjtLhjqbSRYFC2ggdo0SeaNBs+RDa4aJOr76eXm0C2Xa0OavcUrbACO8VGRKpFF7ctR1f/96v5AgnlROWPd0Qf/eZD2J2ahbxsB8B8ohHc4jHUgKXCPYws+CJKlAwZJukJblVugOIEqna0thewh0o5ytDcvOrEndX/GS3Gdg7d/RO8aQjhgxLTldahqwJiXSzlWQIPrEYvk6jabPOtAzxd1aWrG7diePsABdDn03RhFx29li7aKGnj1NfZFIxbW5henEPXagta5CAuRt6d84XGnSwxjJuu+cJ3HTvHgfwkdGXQDeSQDeaQoqbN0GQLiOnSyLNiVxRzz1wptogW44ySdpfUQ3fc237+WhlxIdWXxUKgiZClzAdYZ2gblLDn7AexJH+r++XuBpSJAueRg6V9pFRQIqTqVEqtiTqxdVgabbQSKncGfBSjbYwv3IAZ97wJQzGsnj+jR9HqtXGweos9qKMnYk6HqjNoBW20Zsfwpc/8LfIxPvRbXQQxqzWjCdipmFEBQ2nB9QmQZ99uyXhdvrmGhjEyOz1kj3t0IgWdhLwzzwBTe7HNHB5UhCgoP8rTzI1z9VfNAQwlkgtSalSgzmItJHJxhBJnZJtYaYh4I3AXtuE7DRZFdCexCRRO23LaAxEsTpI0rJqZ5mNZ4qqGZx06obIkPUTi+BE/UEgUlZfUPYligbmEGAC7yYxRBK7mFnsgycS2PnsNnzj+7+wWVG3mXLZND7/6b8wDnWtrs/FINBX6Ee7TiQ2jk4zC3SziEeLrn4n+GVtQipJiG0V5Wlrk00Bec8aZOHUi9W7PKlZtrCmlqE4gdEEHQrpR2TXw3tPwzdNn7khA6G8zpuIa4oTPv5w4X3jdVsZQvle8+ONJ4nSG1bBHrOCClNsAVdRAxejATKFJOa7m4GIlXnqtWbTSv1tHt0sWYzV1ZY964nFDj7wxesRTWTUOgqjaWWBNghFz6AC4pkehPEUYsksujECVQES6SwLGGV3IYOGRNJDeRglSP10bUNlity41uqhKJshhNLuWSS7x3pnVsSbgrpa356f6Taxd7iTlKk0h4xkoO+zfhEiSpZSzKlBOjE5L7XJfq5DqKvxDpqXno2+T1yLwtgwDvzBZ5CaqeBQewEHIzXcWz2KZ2ki1m2qyf937/scVvasAuIpuQcqlWIrIEqxO474uTYWWwhSUDDgbH6e+kskHKSM8K6Nau0MEUm0qU3DyPvWaqjemTl7gomxxY1q6cUD9G/OrZ3pFEESD2bF4m5mmUikhgusD9jsniLmE120wXFj5lg7xtBFD1Aw0MlqlKlVOqkNyZ+hoF09mEYjtUsqItq0Lr3nHDQXkhhITZqLdRFo8H3psMeTv30cP/zZwzrx/cZljfeRv3qLpchNow6yDUIsQwqP0k2i/lIMC3OLiHTSaNS4+eJIJ0tIxqkYGbfgGjJQMEAJ8zeBcmY8HGSQjxNJElaOkAyi1pSzDeH7MtUnF1rMKUer1byqgpzxvokb0ErVNpMJ2BsKTJDKSiRxoCUxy9vRQYp/56ZN2iy0PWumI3XMdx93oJGVh0K83bPjuuHPk7TBzUfLzocefwb/+qPfoRkhVZHrikMaZHExFYsDHOiPctMWkMwVIUVutk5V8yYcvZHkHQY1m7xiNsQ9qq4PD8MD46/TIL2QPjfGxmjDWoZEAd40W6RWH3qlC5EWPHFen8XYUUuULOcd4/Sil5QTtJmdsJw2uU5p46BqwDroIv6ZazD01jdKxXD6+tsxd9N9mOlWcaRTwewlq/D9Bx5U/s9ToTeSw3Xv/yKyhT6kYvbw+H0pChCdcywtcn6lcOhoY6rR2Cek4DVrFvXPDNP1LSwf4bSxGk1kc3kbR+w0zb2BKWCEFhxMobgZSOE0tQKbG7RJmWj8FDPNNqoRMrQAOKSeiCuFVbsmlUaHYmeOyCL+ruOu8nc1OkfyhZwBTAlSp7Bn/rRbqCdeRLxQA8u709li1BLmRXHThkw7WUe5z2ttszbu+tVvcMf9z4mkwV3Az7tixSjeee0b1DZJxpm+2eepafiE7x+XM4Iye55gDHydDmamZ6V8yB47NyxlhlpNysxkEA2LCNjUDSOIhkl02taPVXbTNuEBS51toF4sK2czyu9z2oqGb5wgUtargX/7GTHf3IwvFwNPcUmcUpeM7TeXjrOeFHU3ABKphDZHPJ0QOMn1zM9WDXejHhxUIObr83kR+SXzjVRbOtAvOvBTfOlYBB/7xGcx3RlGNdqLWCSp+6PWFdefDAWIHrP2TiCMJHTopLJ5taH47/9fW+8BZmlVZf3vG+vWrRw6QneTBQYVHRUJOuo3I8YZFUEx66goKDkjsYkCDTRIFgUEkSAqCGIYdRQwIIIISu5cXTndujl8z2/tc273//985YPdXXXr3vc97zk7rL322gwDS+nnlIsSKhGx3yMOoeh3ZPcPtGKfojFqIjTtxgeusFlT04LguRL57dqO4kYP5AAvtTg8TghIDTPSBymoi3ARYPTIDtJBwVpSyK81bPlvr7KRF161aqtmuf4he+HTJ1u5UbMtzYrlv/RWu+0nj9jf141Zg4OTSNs+O+1jX3r/J6yne9AbYJgTaoifR9DCrwFrjaaRqHGaTMCDzDjAJmTZrZnUG4MH5uDJqMlwRbV5B1WElAcBPH5WLkFIcLYXG0rN99JXinxpVz9wiw56CuPGmTDq9y370Gcvv7iaJOyhaFjZeC71YlZUGaUlfrPSSvVhdFgyW7J654uW6wYN9snyQmlbXG9d18uhFN0XD5xwMYHYW3vHrT+wJ558SYYvigS8ad/X2Pvfe4B6jCnfSRAAY5HBA3pzgZd4PNJSxMakwqJL2mgNYCwJ0S7q/rlu0H4R9MFWkgmbnJgUXpFJ9zGhzVL1y/y6HwAAIABJREFUTrN6v9YE701JLZPuslKZweCUtEgZyGNTojDiacm7iQoU/QlHcEWXUqmiFjkw4FoNdpLz7om4cE3ZbEJiABrfyhC9dCepprVyz1ijWVSFgByYlBCvifH0PNsrEDJ8taaNT8zYcSeebOmOfivl97FmGvZTlzSaLQmZBcOPYcrK8xLxNJkhjfgx15/rsFy+X/zubDavWdHqFmVSvUYf+H+JDasObkUScyXMXIkhL6CV2FDBI0YChbsL/3ISfkr0NuUxyoucNyqGh6Q6PTSGu+FRG8OeXAmwrWEsQY2mpT+wvy0657P2l7cdaZkdBm3VDafZ4x/5mnWUKjbS0bTmx/axzlyPffP6222qxJhtl4x5/35vs4P23d/6csstkcxLJZ7jK/qbRN0CgyvkuKJ9qvGBHMebsrlf5TzhcHGt3AeHFMMFwUI5OShqmO7HnNoIuPB9Ne8HNQiXbM1aMsiPKD8C/NAEc0Jy583y+xpwFQAsKSHEBmtNf4jAjfNjVW/X2ru6RI5wLJG0SmvW8ssnrZ4oW7az03JJJ+YrjggjWAmXNWmC6QREDu2pp8z6Kdn13/q2vfTqhDY4HVx8ffKwD9juuy4R8KYG+UxabKRCaOogQvN72jbHKUZTrF+sKDh32HnpGuoVBPoQiuf9eN8yRAmVV7ps6+iYLVm0g6YRZixv1WpDOTSH1yxjzToN9DQ05ARMcV+kN/CfAXZoXRTIKu1jmH6UCEO0E5r6FWJrzErWevsGLJFCsYW8c8ES+VetXJ2wzs4eJ8dkMzq8rXRWDRuUGDu7GRA+oAFt1VLdjjvhRJuaXWAcgaV6d7VCcrElWlnhR0KXpS4CoEk3G4AUDQ3h8JIDE3FIi5zSXpdl8p3WkevU/bglotRllti86/taUR6k3fcY8gANuQ6eJ+Y7ejSxKyjU5QTgBEE15/N6o7MeHlY9jF5EfS+WUvBwEgoK7CbqWQtLu23lPRfYlnt+YYVLvi9v0H3fBbb1+4/Y1I8esblF3db48GtULx0vVOzKm+9WEg903pdJ2wfecZAI7r3di9TMvFBJ2pLh5daX77bezn4RCogGsGztHAkgJBIHQqnB64aAQR42x3owhwSkNBDUnEIXROB8spzrbkUxNRk9dSo54uvyr2EMpNDnbfNxMWSy3FJGCLNz9L2QB+sgU7pxZJBpBXwWXoxQvNwat6W7t0RwTyMrCkDHbCQJAzipXymPAMG6NWsVhbEwmmRLBTA27ao119q6DUi9Wps/fvYZx1omSU6cFmod66tKRwJSLCMdpFecNBLeNxArFH1BtkFzStMJ3BjyOjWuBG0yRWgQIrX2TStXSpYipUh3WXdvh02MT1mxVFDDAqEu6U5P92Kq0daRzlujlrZmnTIVOXbKki244DCmcqEkaNZqJK1Uqemw8nwi4T+XT6nubNkZa6TGLJllVnLShocHbW521lMjvDaeMzDdxMuGmVUq2ab1I3be6gvlQYnkrrxmrX3jkttsrJjzHBcvrlZqB7UQKEDhJEFKB91L3VLqnpfHTeIMldfCwmKfIn2TEVKf2LDy3Tq4nps55ByZIO4cnT0lVYmga8ufPDCmA0TPKog+kCviQ3PAJgh3ydM5isyXI4d1a0EYqDatvHjYdvjZ+bbwlxdt9PMXWa1W8gHXHz/ABj/+YXvmE0dbaZ9lVn3rjtaRzgps+P0fn7Cf/vbvEkFLJ1J26H8ebDsOdlulVrHRqSn7ya+fCMqLQqiUO+XSHfaFD/67dXUusVymV/cFcum9sRwkV6NQqCpUzw2Qiv/UJhM+psS5o4B+7oFwTmxqDoka3mWQ3EJXar6JfVZRUSQIb3DwvAljIFG2MFA7lekUKOb5l/NiNa6TcIuylXJgKBQVG5sesVvvW2uXrDlLlEHCdcA3RRNBJsbfO+TNQmKhpTI/CO/mHl9pS6Nql152nY1PzIu8oKjIzL76pcNt0ZI+AS3VMmNMaPwvWk9Pv0Jf1irqZeu9Ei40KNlWoopAOIH0QH4psC/pAgc+LdGnUYisH0j0GPt8vlOMNxmFMP2PAxJbM2nw6EOZpMUYWGRo8cQcCed7K3SnqQMZWqYaVOr20AO/s6mpiu20bDdbvnilZTJdajKYmhux10JvzBeF1itqKpdCAwkH0eVk4bk3NMKlYV3qKOMMEIWZrV59qW0am1KE9G/veJt94pOHCYD7yhm3WLHZa0lEBQC1WhlLZ7g+b5CnPV4TDpizVKPu7g39hEmIxXFWUmlem2yPn01sXHVwK7a/uXV2TxDDYB3S0J4WgSQXqHY1x1gmwkT7wXfBK6G57nv0ED3E9AXhSwghsXu5bvbZf7eBr33YRn/6Oyt84zuWalat1KhaK52x6V0HbOdrzrKnDznW0oe90cqD3knhIFHTrrzxThtfQFKlZZ2plh313x+3cmneRka22s8f+7vVSGCouQUADkNy9Gc+ZP0D/SpBqLUrge4zfOOSUNcowQqIA7qraXoJDh3IZNpaVY/5+X42xxBqJ65kssiXcvhZP8JuR4Ep6WgtABViCCxEPkjdaJVcA8tbCYPUjvS4XNpFggPNhm3ZvMme/efzVmnVbLbARPWmGFYnnXGMLVm21IaGBnWdAvqkEBEGlyn4cjCwUa/I4HCASWXaoEerYasvuMLGJuYUVcgAJxK25pJvmCUrVipWrFIuquXP1RvrXquVfKQ/b0UW8V5DtSK+fyy7qQElGEepVgRsRfcYSl/CAEI0wH2o9Bb0uXU4SUPCVADQZxEUQq0YOVRE40HUWXOEzhFWoL570YVX2eZN04YIP4CVcI1Wy978pjfaRw55V1t0XDKv9arQZxBjUiL0onxNMCTegJJN422rNjszZxdfdoPqtRiQq9eusc7OjD366ON2y3e+bTa4r5XTSy2R7LSmDqU3FERD53xlBUHWEM8Aznc4i4jo06sF15oDzjVv3uk9LZgtCmEDDUBaSm01gqDIGObCbl/XBVSIobSTWNw7RQ6o8rSgNuBaVds2CWB183W72ZKLv2z1xXlbf8r11nr4cWuiHs7JBNxKJm2yp2W73LPGfn/lWut+80orUzMLnkSDnusNu3jtbVZRIGe21y7L7D/etp+V5mbs4f/9q03ME9pGzVqTNTv9a5+1VtMbDBQ5AAjkctJIjhxnvBQHUOUX1au91KB8jUhB+TxgCG16jvyyMVmfSLrHKLCJhJsjiwrpQU7ca9gCIeH/8vfQOkk47fvVDzC9uL5RWlarLNjzL75sv/7V0wq5sEllapbNlh1x5BH2uje8wRotn0b3///yFkG8d0rv44d32yRB1iGZaNk3zrrYpmeckM+9otB54XnHqwcVcKi/t8d7mBvetxrr/qrZB5X+uCElBk/Yx9wjPLV4uH5YolfTBIJQEhPfuwpiT4Tns4UiCBijvIijRDIHNWzX8Mqonu31bmicTsaQvG8I4zHMZ5xxkVUqAFYJNcNw+EGM/+tD77bXv34n6+vp13NCk8taSOs6FRUGkz6bZ0GRJtT3wQF434VCyZ57caM9/ue/2gc/+J/2tgPeaplswi688Ju2dWSzdaQ6rdq1yuazK6ya7vNGnGDoVM1JYLS9RIaFVfOKhOadtAPSzIZRmEz0tGW397dU2lGZxEO6qObHxtIhbHioHBdN7p3NEaQ6faO41i7lH9BILaAGbLUsn0haIVUXwpy1rI0N523n606x1I6DNvO3F+wfXzrfBsoJ6yDcTDlaizebt7LNZLO26q4z7YU//84qNc93/OFnFK7NzEzYP9aN2b0P/14PIJNs2pGfOcxymbr99ann7HdPQ1NzwEglK0valz9zqK1aOqAGb5DcwcEh3Tebzw9MnLVLmQrShiPpURfa4xsvX4kwobEbnrtiqWmfYwOCYMuC8qlhc8awLzZpyHNrTKWLmwnND03aMUWJ10bP6sYN6+znD/9eD1Oc2kbLyvWavf9D/2n/9q53tsPKWBVo52J054SculGc87qr5uY4SAcVMZlu2WmnXGAzHNwUYFXN9nnta+zzn/1ooDnWhAADRnHQi0VvZ9REwoWFNuIdUXBeV6b3NsizAA5JjzuE5tG4xDq5YyUOXqkc1nA5XJEnQsqFkwF0WrR4kXdKpTM2NzdrOcpDon0CInUoraEWy570mnenAKTTTrkwpC2OHWBkcQDHn3iEDQzkBGIymRGVDQxbjJTm52a0p1XHD/wDFxwEXUcDu2StTIdSld1228tq9YqcwAknnGLJRsu6u1E3SdlcJWkL2QFrDPyLNRLeiy0pJbfVIqwANMpwJiCw8HlEE+TB7ky0h0Zf85/AAG04P6KlEagSmpbyZBzrIxJGQD2jNZP8SMo3Pkajo9qyUqppKRQsyM2olQ50Wd+h/8c6Pv52a+Sy1nh+nf35xDXWu2HaOgiRMklJ1TToP1T9sGXVZMPG/nWJ1d/zWsnAuEay1495oFwrG4b2tkd++yd74rn1eigrhnvs0P/8d2tWq/ade/9HCvCx3xVA4F0HvtH23nUHW7FyRXuwFpZfPbsingfeqiyrh/o+jdDXKW5MdVKJk+tKDIpZAlPLJ+wBvhASbScuH9IQFp+NHME68jDE5eSJ4yC1MHlBZQc1MSRt8+aN9qN7HxaAwUEEZClWy/aGN7/JPvOFz7cxBO2D0Jboid82AKgyP2OVYqFN4eW6kbKZm5+y1eeusVIZTB5/nrKDDnqzvffgg5yjWy5Zd75L9++dVC0bGxsTe4swlwNIIwYGNWppd1ALRe0j2+GkmJD/ekNBRgeK94pfhPBKDXgeQWhBIX/CVEJiMBpjVYRIB9aXk/Pxslmxqij7eT856VTDyRnNhgQWzjvnCgdnE16S8464uq0+/1SrVGbV0IEoHNMPCaHFvZc6p0eXfG7/4IDNzxeUg09Nzcgrwo5Dfobcvb9vUPf76KOP2YMPPiIwFRwFeqeUK5Mm9tTXTz3Nnnl+zH7+u2etmuxRyZP7zFLfFo+acBlHiJF2aqpKhOyxrXt8UG42InyxHuetWWF2DhBjyMFizushoqOf8soa7NywCt4tlbfGULelX7eTdb/3QOveb2+rZxNWL8zbyJ+ets1X32d9r45Zg+6UVMsytTDs2qOENkd6pitplSMOtHKiYnXxNgHQOLx+XRC6YymHDpNLrvq2lZuEl2Zf/eInLNtYsO/e80uroiKhPl0ecMpWLem1zx7+YXV0KB8MaLKoiiGP8dw9KCuQW4mM79ROHz/p+Q7ibz7Eyr0qG9jZWA68ONjgTQmx3hdTCT+4/uVGMciqBE8QsYE445Ue2OnpMbvz9nusWfPaYZl5Qo2aLVu1wo478QTPo8OwMJDbOJ+Jkgj1ZeiD9QpNEOTyPlyK1/f09Nr4xIgf3FLTWkmogg372Mc+bG964x5+YDS20g/cyMiILVmyqL1+3HdsPyMHjjREMmuRIljj4DW3XwcOffTWREDkjJHKiPeNzkFSMmGWkFjeQWxO5TFAPRUBhNK01TKIIiCqCJgSaSNvxxx9ZqjJO0OKEg+G+vQzjrUEWEeSCAK1EPSrnRG3bcZuRc+X+49RhI82wYgmbL4wKwB02bKVVpgv2SWXfFPItvSypOjZtIVGRVHCRz7yETvgwP2UBnEQy7Wm/fXFMXv06Y326pY5a7Xy8rKNZMPBMHXree1ZSP6WPT6g+6UpQPUkTS5rqd0IF69NhwIFAARehTfBK6FG0D9opXzScsO9lt53b0vvu7P1vWE3a0JHROkBAGTrlI3+5Vl74eYf2cCWCUvXmpbBgoiUHtkgnuxHaZLYjTT5nl1t+rWDCr9J2Fl8wrLYi6m+23TW5/dIkydpN996p+2//wG2bLjPuvId9sivfmMvbZxTWx4sp0SyaR2plJ175jHKVfEO1PrQMJYqY8aBoFhjxkPIy6sjxkGVTJDWRLMpJ3kWz1lbLZeEAQkFuo/AHd7AvbUr9XMgvfHCQzXPD32wlw4j9cFORxwhDhB68/1KdcFSiQ77/f8+Zk8/8fcAfDWsSG0y32GXXHZpmDcTR4iGubNBwRLomzzXieh1q5aKYqoRTUDIGBndYFeuudWKiLgHIbavHvkZ6+/zaQYeaTCipNump6Y0FnN8fMyFC8JYFU+pXF1C9yvlCTfGiA9EA+b32Gld+bzNzsy6sEGpqCYPfhaNIx5GgntCrr27yc27A1QKH5NoeJUsq95hNrP/DmGlS/Y2rb9/wDZvHbXV513Vlqd1XnvWVq1Ybp/93OHaG5AcYrmLkBnecFWySt5LrnUI/bdxSh+lrpjrM2iMa5iZXrDrvnWzJZNZGUX6zXlNVbX3nJ122slq+O/tdVGFqenxtjh6odK0YqVp9/3qeXt+S9GmFlrWQjkDZU6xv+qWGNnjgy1CMMJJVIYWmg1LQ+1LmJV6MpZfscRSb9jd8rvvaLmVSyw52G/Jzow1QOUysEV8kjj/y82WbeOTz9qGX/zWEk9vsNx0yTLFqjXSZpk6OXQ9dAGR7AddWno7s3SZBMoknpuSSm/Wip95k82kK9JdwjPyoFm8uQLMGTaBWXffgA6Kt5Wh0le0cpWQrttKxYL9+S9/sz8/s6mtbkC4lkulbPU5xznNkFJFBklOZzl10zNbZtSHz3SN+SchICEX5Q/Kz4R3YgIVGG7sWldcKCwf6S2HDhYMDRzwKFmjRosgi+LSrp6zcCgoNThzykN195z00GZF0MhSOrOUbR0Zsx/cfo8sOb9XrbZsslywK69eK/pjDOXFtQ3IcIUh0uWSIgcpKyh3Z/zGgkLCeq1iU9NjdsXl31EDg2eZSTv55CMtnXZ1TAAfNQJIZM37ZQuFBa3bkkWLdI08lwLicFLmN+Xh8sahCYBDENVBkEzlIGfDNEKEyksLBT1jhrSNEoYDOIn5tU0TTOURFDxqNevt65PHJiVD4havqq7aIDKPfI5SmUbTXl6/3m6+8S4dZmq3KgV2dNiH/+sDtudeu8i4w8FWGsOYmS5C4cmQLjniLYMRokz2zczsjOfBoU2UfURU9sjDv7G/Pvl3HUxNWgy6VGTNr33d3nbwe95l9TrGpsN2WL7cJiemvZEeIK9WtGwiq8aCucKs1ROdNjLWtJ//+Vl7ZbRu89Zjicm7H2hl+rots+OwZXbocxK0OvcJo5qWZLQDOlOlqhUnZqw4PmGFZ1+16rqtNr9ui1Vf2GT5essyADpYA3GAE+qrTVVduUI8ZCB1SbHAYnIKV8yXQQHdUnqiPtOTsspn32YLncyLQYXR66hsHhXwo8wLaHjKNWdzHZ3KK5B5RWVidOuIVYolW795iz34iydDkd+nHCQaLfvmxWfoUPK7CwvzwSPkdIidoOJhr8TQOVzBa3Ko0VjicIjHvb3MrIZGeV0T1DSyn7hXCbABPqElHco11DhjmByBKZHVU7mgtJgXM4rrUSN6kvpx1qbGp+zG625p85OrlYZNFgt23U3Xa21iGCe5sEACATBsVEGSg/QJoTlaX+UFKxYWlMNNz4zZVVfe5m12ut+UnXHmcd4QENacziLWgC8iFbwjBg0pHQ4sX52dNEl4VEHLJlEN3pZD4ioZfvDcM7fkwbhvgUWZtA42/8ZYi0KriY7uob1P12ca43HRv8bgOSHfQVS6wHg23jCDyob3mj/x1JN2//2/CGqWPpWQ8P70U08ytlK9XtHBJWTnQzNpIqKsTU5NKoUSSxA0GK/ZRe5e9AaRQOGN0xtY/8suuVa8AOZE8QBJigTCZdJ23PFfs3QGz+nenCiCz5EKB6owRHFBuB5RORDnUrloOaLBWkrhf2Ju3dOtRKFszfmyFbaO2PzzG2z2n+utsnGTNcamLQ90XvN2JuW8tGSFso/mnQSqIIOs1QGDtwn0t9gGFSelCUmNyhPqg3RVBcKiTpC1tNnL6ZrdWt9k//3lj1oyBz+1oBwml3cAJDJusGoKM7p7dCDiYGEeNCijxHGaTXv2uX/YAw//2SoisGdU68tlknbc146wFSuWtjVx2QnaJELWyUfTVizhdX0mTSQ16MDCOop6VMGbxFolHgwAAtlOVSbaA5uh3/nnx+kKeE8JxakU41PpIRiwebhXjd4gfWm1rI+pgPB+az6i8/qrr7VEM2nZdE6o6VRx3q656QZvRQylJZL9tnEMqDYHq1YpSeGhiQepl2xiYtx6u/M2OrbVrrry1qDVxBpk7JjjviSkXrV9zQRyCiiHj9p2rL2io8XGXLJkiU1MTbjxDqJt5K2E0vLAGimSF/WP+wYU09CtZErfx3vG0lKt7lMN+Wx6a9nc1Mw70WzSHF6vZPjfnf/b3d3lhieTViSmAW8yFFn74X0/tl//+n8dmMphBLxF89zVJ2ssCXk841kgzfC7maR3xnnpzjW2eXZ9vd02NTWlZ0sEpucnkgwRUNNefHGD3X3Xj+VICO9pKPAGiabtuc9u9vGPHyrwy1NPP08Ab3FWcmSjOcbhyqS+5kgCe5SSeG6PtwsKVfse6ozUEUVXdM8oUCGIyIlYEb6ilKWHZZENtY18gcV2fSHPdfiSWnxoKxOoxWGSQkHT5rIp+21y2h7LVNV1ctzXP23lwoxyP5DCyelpdYSwwdkkbHDQxu31o8i5uCnQTz5306ZNCqXuue9X9uK6rQpRIXV3pBP2mcMPsX/919fJikt8K1Abe7p7tOHkeekU1fDk7YTBlB46M0oWMqhO8Dr/ooxCCcOHNbdVNxDOzuVUQBe3JzBj4uKomSMYxO4er5UK4Q80SgwDh1bheXHB7rj1eza6ecxy2bzyp9ly0a6++QYrl/zBik4phNytOmR4WX7CZO6rUra56Rkb6u+2mekJEU82btxs1157m8+HSpjE3b961OfE12G9o4ER2URytH6v8kKI/pUrAvyQ5CFHdxpnwuhKwqty3RxSIeSphO200yob2bpVLLA4VMw1rb03Soqhkjjy0ZzbaKo+xlPU1bBm8IsLCz5cnIHogHA77rijQl0OELjNjTfcbM8++091FZGeYYzz+R47+9wT5Ol0LyIh4bmzNjc14cZCpT0veymCiXTe0LvuP3fmE3nyfff81Na9ujk0X8AdcGNKmnH8ScdIXkh2MJwnnlds1pCoXWjMiHs7dq1JXIEvDu7fd3l7S1aFsC/U9IDO1U8r+UpnSMnbhhm4PhOU/CUucuhOidKRQdlBnxFqwRqiFUTW+D7vV0iYbUxV7c82axtyLWuB8taqNl8u25v22MkOfPt+uiHCRQgQ3CAT75jAjuedmpy0TsoMCcJaNk2XvFFvLzKkjNPskKLjn578h11z/d0CJeh3xOO+86C32CGH/Jdeo4bqQCBwEAjrTtO3o67Sygo1bl8PBxpUXwxsp8ikicin5sCGecB8hq83qDRtW2HMYmjUj6FtDGtl4cXEIkzyMN1HZjiSzAb+1c9+YX/+wxPSLyY8nq+V7AtfPcL23nufYFSo/XmPq64tWHYRSAANaxWrV2rWrKF1PKcG/C1bR+3SS66VvCpe/i1v2c8Ofu/bVbNeWCjKiGZTaZuemRGxnnv0JndXT6SWyWu6uvOKFiIqTq6D2J4a+ANnm9fxO/wuh0jN6LxPB7N4UbtwkbyYctAJDnjFmvhasx5+cJU/57tEOxSpRs7AmzHUxighw7RdftkVMk6u1AEWkbRlS3ewI7/+Oe0Xyb2GUidhf7JJia7Te8nTSf3J/YpNTg7c0+1lsXAu8p3dViov2FVrblTLIt6fL5whTm+XXXaxQw77EPRkPQNO1PaOh3uSgQ57UVUGxoeKiaeub/f+mOAnV+wvBQyNDNmuTqlDGw5mRNO0ELh39ROzeg7wYVFSWB+K62yMhtecKImQm/Lgs8m0zTYqVutIWWrVYivsucieWZixB37/uKwPYIFarMIcWcCco796uA4PIbl3eqRs6bJlsv6O/BGqzCssZTMPLxpqgyIgeXScIEX6ysYNdu7qa62JymDSB2qtXLXcTj7xCOtI5iybY+yDK1q4z0zooWB1NOM1rIUsv8Izn1zo9V1XamANfZN5eAXgw0NwZNkR8RgWubfmMHmOGz1tO3pRLdhJJuoECaqP4q4GttfLL71sd91xr6WYUl5vWalet30POtA+efgn2yUUNTyEkp6Xspz9QxkOnrLVncIIQLJ164jNTM/bNWtv8vJW0+wrR33ZBob6LUekEuIJs5r6pNUvqwPheeXM7JyQ20gsiQO4AXySrIU2IdEAtVWXtVUzvlKUvA5ftiNjC0Fz2mv52wZno52t5pagEaWy5XaypdK7Ar+AaqoSl6tYoMpJOMuzuvTSK2xkZNQVP+T10/aW/d5oH/3oh937yXt75KNUp4bCSF4RF3I/7DkcCRRNwtply5bbxo2uQ6W5SY2Kbdo4bnffdb91dOa1z7jGBdDyjk779KcOs/7hPpdI6uiwhdkZvYb1Y9+7MD8sDJ/J7KIPoSQLkh0ObfvgeumD2l0gGQQ5mfbBDQQAWQNCXWlMIS3kaLQCZaRbRHxvWj3RsGZ3hw5poydrXTsu1t+ruy62Yp4e06QtTM9ZpVy323/8U1kVeMOIVZMPiNFUqdgXP3+IDfR2WblGWJyQFacPE4V58kg2zfTMhKw23+/M5W10dLQ9e2bz5k120IFvs5nCjJ1x5hqbmCyo3MB9dHXn7MLVp1pvvkfavpoWD8ocvK3fO0iqN1XH/IwHyn+RqhgPrkJdqX94Ez3kBCeLeHPCtoPrDClZ0TAwTQIFgeIWYiEPP4M4t09m93wsHtz5uQW77JI1AlDUcNBoWe+yxXbGmWfrWtVmp3JJLEU5G00IbzphCzNTVizMyIsNDw9pzX7/u8ftlpvv1OGrNZt27upzLNvhhzaWSBhDRxrQle+yufnZdhrEYY8jVLlGNjyhJZUEvDkGItFsiNwwPT2jZ0Zk5GQJb6cEwALRlv5ZKMl5bTuMlgxhMT+L6UA0hrl8t68nayREPtS5ywBOXgM+66zzbG6WecKu48R6nHTy8bbNwWmqAAAgAElEQVTHbjvb2PiYT2+kbioEuGEtkPhwPaXinMpy3NPs9JRyV6538+bNiuqUE2dS9u2bb7NyyaRdRaQoDKBRs4HBAfvCFz6pzq/ubk+FIndcVYWg8SZCShFcB/qnt4xGFpw0wMKA7sSTK/d35hT/C7pRgme2G5YVaV78EuPsherKEzSsmEtasi9vM4MZm+1MWKMvZ4munKV7UCQEmnc3T7jXSieso5W0JkwUelvmS/abR/9s6zZPhPpgr1WqrrqByv5++/2LHfDmfUUOTwf4HlTW5VOj+FjgkKYResuKuQNwwGKA6BFi1Vslu/CSG+yFFzaKLcRCQB6/5MLTESG0RDpq/3rYFVMBGRKQbMm8OpLpBBXnJgtICdPzZP2V6/ng6HSH82SVF0ZBdhD3KNcjHV5y3RD+BtJ6BCZ8j9Jp40oeYglJRdEbJiDqX/7NK9XBIpwgkTJY2ZddtbZdP465UvTokigNk80b1bL0lCdGt9pAf78Oyy9+8Su7796HZEQofFxw4WobHO63uXkH3Pj9DjWsu+ffOjqqTQuvl3VgPRjclksnbX7ePTAhfnFuzhqAKxna4jyEZeojXkXjV6gpKyUCw/DSGOuIlxUoKgka9lAct+kgl7P5/J6kl0bomWH2jk9713NGUUTPqmDnnH2+Vcre9+yAUtouu/xiGRfRDquw8ZjMkFMoXFVJ0D17MuGcZb4Qkfd+aq+5x9IXf7/xhu9IUL6js1v7gSiO/fXJT33ChgZICXx+kaobNKyEFEZaz6HfV6qkgVYcS4UukO8OUljNn1btTzFGVrWaBJpPqkgvACKMOaynTPKoGbxfZ8LSOw5bZcWAVXqYMNC0Enlp0JnFIuFBgemxQjQnk89I+yfwnRU+ohvVqNvk5JT95IHfWJ2ByTnGUThyCsCUyrTsy/99uAAgWtpU9gHgSbvYF1azo8NHHPKzwWFU+BMmnWg2BS1lTXpgG/bkX5+ya2+8y8OrdEpDmc5ffaZlMjWf7RsOXDLrVEIeOkwlQvToIWUs2sOsIdlT6vASyPZfHiIH30mdMhA2hH6HAeGANF0AY9IiJszzsJqNKHazcno2Laiq52SIrZFSeD9x07598y326qsbVQeVbEAyYZdec3V7M/D4I5LP1cQcmmiJjQzIt3nDK1ZamNdY0J8++HP76UO/0rNHB+rKtWsFVM7Ozckjo1jB78SRK+R3ceNFD0hqUi/7QVe/q5kMqBpCirOiHgqdpuUTAQMqDYp2+Dc9q573aW5wkGfNh1nBUs9QJxGlFUgyPgiN92Y/aDhYGPzm+sxuhAnrp6dn7dxzz3ckmoMIut+RtYsuOl9MOxpNpECCXnMBbe2MJH6IxNi/1JcVNaEXXXO6LV/sryg88be//dN+8chvJHkjrx+ihaHBXvvoYR+wTqIXqZsglMeM3EhqaVl3l3tz4R3pjMJm1fzDJM34HCNnPvHHnd7cwtPy0DPNhC1Y3aqZhFUHOq1/r50ttWzQios6bKZZM+vqsJRKCPhLn/ZO6xGAUnFmTjfCDBUAGG6SBwBXlUXhQuK0MR2erIeCExMT9rv/fcKm50loIIZ3akwI1rhaL9tZZxxv1qhYoeggCP8pf8h3yqry/s4VLdvKVTvpYKmpXZPbQCPr0oJCauTo486S5ebmUfM/7ZTjbcnifpVFWEwsp5DYdNqe/+fztu8b/lVhqELHunNWI7I+PTOt2T+AYpE2mZVkTigBCb111g6GUGUwjXRxcEHzlkLfJz+LpAQeFrVr79bi4MY8mfAOPSQUIFnPhP3pj3+xe+75odg+tIpRq117443tvBlvHRk98br0WVnXqtq8ZbO8R193p8Cq226/yx7/w5P6/XRnxk465RRFMOwN6qHkwXEEJmvERoNGOTMza3vusYfPBgboq1VEzKDEQTPDYL+TZGCW8ewJOVkqjBesN6K7GBoDAsE+Ep4SZtDyORFoEodZHGSK+97dJcE5rpnwVwbXx5FieNl35KCFhaKdfsZZDsIS6WQyttPOq+yYY76mKIz8ER0pDNj4OBEg+6aivcs9VUpFb2EEoKOVr1jUGm4fyn/rmpusXKyLp43KhWZEJZP20UM+YCtXLRWSrxwWOR3uLxBvyHdhyEUBOtdjdsCP/aIDLCDO8ReF0D//xCEtDqmhDtiXs3R3p7WyKUH7XT3dWox0i1EIiGjCrmqoN1HaRaG/dH52ToyoqExIo7dCmHTa8l3dbe+NvjEbnwslb9V8n0TCRrZM2e9+/5RALjGOArm8VK7Y2w58k711v9fpYLF5RLKoVq2/H7JI2nKdPfJaGJHFixZ7eNZqKnf76xN/sl123lldSRzcY084x8pIodJHm8nY+973H/aB9x3c9m4sipBO6o5SE3QtJaGjgafsltZDajYbQnGxtxS0efsDIotMbTvwmmWwwgQ1IdUB3o80Ov1uQPCrNe+KifmNpD3xEhm0f/PWnc/bhvWbhZSqFlqpaDzIFdddGxQPGS7shiSGlfF6+O7gwKA8VKVcsPmZadu4Yb3dccf3VYME61i0dLGdedaZAlbmCgVDXoaNxf3iDWP0gAfmGivhcPmwNUf0ObxEFYipwWQDvOEZahpElDYys6WLh0SiIMWhTMSG17jJYPw9WnMRPkJuIiRI/YpaNMDc95rTTltieLH5yUHZXzxH+mVPPe0M77flNR05e8c7/s0+8MH3e5seTQjzc0oFXC8Mj1uRMdLhpSxYKstg4JW5Z54/pSUiBwz5zTd9zzoynS5HKxS8rNz2S1883OqNsgw468PaCMRUq6x7Zp4vh5k1rtBRFSYVOlaRUmqnUme4hsTdV50gVDnmWq6P7GR6nwgeWDRhrqjC0DBqMlLAiO2xevwZ65E6BNKHNRsaGvJJbqGJXu6e0LzKFPaWHvAjj/zOKlXCVAJF16SqVetCHo86+tPWCrNyya+XLFtm1RrT2wGuvM7a09trvb0Dbs3xbI2GPfDAA/aOtx1oiRY6S027/Kqr7U9/edYyGebpJuwtb36TffmI/3a1ytD8r4I5qJ7a9OLwMsZpOgMGSwuQoCl1msCHd2H+q5MouG4HojwfkuVvxfIPyGWwoGrf2zbdnVBRHTTybhkh4gJhNNoyFMI1tCorgkAuD/GkaeecdV7IP/01qy+71PqHBkNrpQOlMe/2afF1MaW4xl133VVtkYBGk6Njdvmaq2z9xhFFJa/Za0/74hFf8p7QdFoHi+aBXKeP3fBD5uioDkJob4zElMgG0kFGqI/QmQYOt2xG+BtLTGAlDgjVrYqGV5D4ZSN3d3XJ6GYyQe5Xapo+j2lsfNzXDGYZ1Cf1EGMQzdcII0FzQb5bA9fOOWe1vJy8cCppRx51pDrEmF5I9MM1k8viff05IgnQtMIsA+U6bWZmRocMCdresM+Q16GL6re/edQe/+MTCnmlJ8UggEbNPv3pw2zvvXe16WmQeL4f21aJHreN/4yht3L60EEmkC6kEBhOTZlkgDhVi/uuObkVw1qFs6F1T4AMlEAU9rarAUoJPygS8HssUHTnvG5qckoW0KmECzYwNKRifDzQcVwjUphefmlpmNWr6zbbU0+jLuiWqMyhltSF2XEnfjGoaTi6uXjJUt00KoPk1gIzmi3r6xvUweUQR34s+QjhWrVcst/+/jH7zq3f10hHCuWrVq2y8847r93gz/06Z5q65YKsMNQ28qVysabQT8oP9Zo2sTYh4Av86HLRXnrhBVuxYoUsJyGfT1v3QrsAIrE6nSmjNY1lJrxPoiUghTxLXGV5fS/bOLnDSzTpVDYwqqB55u3Ms86xwpzLw/J12nnn2bIdd0Beyz9bAE4YKRkIIXgtrpEQdGCwVyDMb375P/bjHz9gY5N0ppj9x3vebfsfdID1glXMzwvlx7suX77UXn31lYAB4G3CoLVQ22ctZLBoZaPHN5SveM+a6Kt1l5RVe1/Nli6lvFfQurPmZSbC5xgxilF34CmrAV0enemrCXhZsE7V2hvyiqD/aooP9whyK+yDWbSJpD366B/s7nt+qGgBh0LIf+FFF3o6orDa07CFwoznrgCkC3xG1hbmZ6xRcafE/TJOBoWVQamNgOmYXXftjUL2yaupS6tslO2wo4/9iiRtOSORLgu7bHx8XPtGHPcAlnluD+rskR4YgqRZG6RSOT0v31tpS/zoutP0xHWKQ7VOmyBMPI8oq48/SFilVG43F7NIGkhNrYr2JkTWVOf0dii+D9sp6i3zQDSqEgHrvC+oUFRr2dxC1X7y40esWk04Yi3yPCFVy17/hl3tfe87WA9d6KqEV6HI9Vg6l9UNUg4CyYtJPIsDQV2zS8slhV8s1rHHneyT0TNJhTHXXHOdX0NonueAsHj851I7XjZotpLKQ0UwVygPcJBRzy8US01xD/kQy6cWuJCLcX/R+6YgNwSryibyzQkguC3MjkCPb0Lvc63VaMfjetzjduTz4rR+85uX2+io0+94/eeOOMLecsD+Mn7xMPtu3/ZvnmE8uJVq0cZHtqgDa82Va21yqiCvdPSxR1tPX6/kQjl8REwYLs05azo7jY3mU/x8OgCRi9ZfIuRueGK4qrpk3YXLBZIlUzrAgGQ8b9YYY4j353mR/ij6C/OdQKNBnXm9lESCogp1eQ4uho9n7FGiYyUut+vo8f0//In94pe/DtMinGNww403WKm4IGE9ACmuNYoDaO01+QJJ26rVSs5LJoxm5pK8ovp6MTglu/ZbN1pWoXnQA6vV7BOfPFy5LXVfnS9IS7wnTADx1h3gigYpEjA8vHf6J9zmeLAdJA2i6D/81knbBNFbXjNTzlKtiazvVoa6GjWlpC3Mz7fRZiycgw5Nq4fWJiXRKbR0nUYoRJnp9Wj+hG4QaQdlUQsoaaI7N481ee655+yfL4xatZ7UhqEvMiJrR5/wFRXHKahTKlWfpoj+PCSGNBesu7dHh8sHOIdZP5aw/r4+bRYOwKc++XmrI8Kd8qL5TTfdFBbc5wBB/YtKA3h9X1lQR5hAgdlS9fxTOUk6pfyGdYNcHz2OvEoYiAaY52UD6rEgvY4WIs7m5Y5Y4nEv497ZzSgally3jEmt5DlzKmX9fUOSaHnqqafse7ffpWfDfwe881126KcO176OdNNISfWb8UNMGAioRJfQxNiIjW3dYt/97l02O1dUnffiSy9VZ4/wCKaz5/PKAbu62JxJ/RvyC+5ZXOq+PkVnkDMkSBBCZ1B5rrcQFDK4K6UjQbxBjQW0iBKtTU2FpoqEDQ0O2uT4RDst6+/vtSnVT71dDwNOvk00ghGgzZBGh8hdJtyV5yIlq1TtqquusY1btjgwxXiXzk67+OKL5QyY1xv7XKVlVnP6Y2fe97eoljVaKoOkU0itYh5//w9/ZOvXb3ZkO6DW+a6sfemLX7Levm7tEcn9CE12MM0bKraNo+G5eoupH9QIAkr5cTuGYvx54t6rT1So7EOjfAHFvcz5MGtHvJj76pYB3Vt+zmHmAfBhqqSQPwmZTSuUxDrr9UFMjAWkQO+slIoOC2WGnm7mzXpozWu+e+u9VqxQLvIcG5Qaa330cUdaR44aoHsyPodwiNwTj0sNjIkEg4OUn6DN+dgJXouxIc/m67zzLrBn//GKroND/oMf/EDXIoApCJe7JU0qf5a1C6oDHFxnS7EYgSBOe5tANi8NcB9x3WL+F8svbsx8IoTYVCHfUXmMhxoeGmkKX3pg8pQujIekajy4IMmICuB9Vp9LyOcHvX/xMvvG+ef67wcOefTwsV4vDrCZjY2N6v0mx7aIVLB27Y1Wrbm863nnn2/1pkcVsSdWWEgKI0uI1yHWFsZbpUTyQ6YFhFDYm098IBpeyimOHp6LeBGUMMnbMAYYAg4/h1czk8MIEQ938eaO+rqQvKOrGhpGDbhSUV1YDKka2ljz4qjznnGvnHLy6TZD6EnbZSplb/zXN9rhHz9cCPb8grdoclgKc3PtqQmkPzwbPc+sWq30rJUDlwDQEAJs2IUXXaLuNEeJHbR898H/x/bYYw/dWxh0IgfmIvnOVch1ODqtMlgoHUXHyWeKeRV42yoTxUkW4AA/vv40HVwv1nuNy7WCUGrfNjdIag4wi/CaGmhNw3E1CHr7DF2Va5Ipm5mb1aLNzc956EKY1dfbbufiQM3OM8LBgSRR/SgJ1Gr26ONP2LoNE1YLTfuiM5rZ/ge91d75rrcp+S9XFrRZevv6pWkVwwfCiojETk5O2tDQsCiOcDCx+Ljq559/xdZec5OzojJpO/PMM+0t+71V5QG1DYa8kzXx8ZGOMjt44iwf3q9dZhHAFLS6aPRG/IyJ8YwuDeTzapm82FvL0uHgAn6p40gHFAzUmzH0uRTbA9E/Ug3lNYPkKb9TZJJ809Uy2ZTcj9Q3Mx122dVX/X/qqzwvv+4QliXJp3P2wgsvyivNTI/bKy+9YNde+23xfTvyHXbOOeeoIcKHbfuoTJ4/B5c/RdmbR6DAPB1ijnC1IoMtFDuUv8AHCGWjvE3M310s1nNwiBaRaIBnivxdZiupdVIhposbaFIC/HKh0i6orxnFjYbKiKw/xgQnETuv4CMce+wJqihoHEjC7Jijj7HXv/71Mi5TM5MiXajxo8kAbHdUHNyobKIeayKnYtkG+7q0z0g5Nm3YaDffdIt15XtEBfY6f8OOO/5oH5fZpPfcjS+/42lZMHA5Fw2IXnR7YEoOY7upltsaDvyeEw/edLom0vNUeWgcRh5SpeYgFDdBmMvq4WFBxxYtWuzspECtw1I6WuZeyEsk3iBeXPDal8acNCBtw/0sW6HoPGIvMZS0gbjQdes22q9+80erUKZrJKxKY4JCtqyddfbp4tmqnzPwgBl1QdM1G4LWv4hww+jRjfO5INQoBtYrNj251c48a41VkNbs6LB3vvOd9uUvf8XQ5/Vaczg8gWYXrSHXuD3yF/NgSjryyGqccEK7AJVAT8N7VGtlARNqzIfJJaCFHCq0SsqaekikyQZi67hahg+q8rAX/EejOgFkJsfFn8XSX3zJFTY5MacOFkpGV1x7jVNRG4HrGmYUsWEIDZkRBELK88Iw8iypp6+5/Ep91g477GBHHXWUJGzdw2+n0ZzyziYMrufeNevr7bPxsTGV2DD6TlsMwFU6LU/IYRG4Qm0fWVUiGiKikJrJE0lTmbZMP+jkgLCylENnsoqaRke3yijy3FnnOC4Go8rokZg/I2DOvlAE0NVjR3/tWCvXvO2U91t9weq24By1e4wCXABq3KJqUnopLrSbIsQ6C5GKxuWEkPu2m79rr7zySpjc58+PMtOb3vpmr90DPtW3lfboN+ZecSzsUV5DM76GnGsfeVeUkzRcjCDiIE4KImopWuL+605qyVITIlc4wB5+IE7FQxMTRU3AziJxJoeLo8F44cN5KpAG+IBY4lHZgf7SojcnYzUV3nZ1e100gF8R/QVM8k00bb/89eM2OVmU/AudFa47lLCvf/2rQoMXL17i0wPZiEHrSXlXl4NTkZjNdYs5E8oWE+OjlmiV7fgTzrPZYkWh3YqVK+3yy9dYPhgO0Go+j+ti80Rks81cCSFLLF+ogyhI18a/c4oBkCJ3mZqsE8QJieGvIHRmVik6F9WNg3teR/C15GFwtkdBrpTh4SEHpjA5ZoXCjOqkd/3gR/bM35730Y8dWVtz7dWqxQauR2CseY0TA7l5yyZdmyRiBC6lbMvIiJ1z9rm6nje/6c32mc99Wt6Wnmc2itrN1CEWdLe0zgyy8kFvhbl5eV5+Z5aQlAMS5hypw6bsbCOMuLxlC0ZVT7uvNYJlvb39CpkRoQMzYM9QNqJ8hJGP4evGTRt1L+wnNbS0kK/13LFWQ9cpTuZzreKTTjpNooJcE597+RWXK0KQqkqomqhvJmA1Cl0hFgklJyWpKIoU040DVfcG+gvPv7Dd8+zD3lp21tlnW61eUkO/UPXgiSXXm9vGw+bCnJddUelRxqMEv6Gse4vpHPfP+/I92HqS8OXgikwgAGTbgOGFEghdWtaNeqF7gzC+IsD09FjyPW6I8gcfIP1gkcC9JQtJDh2AVktkdulM0UDd06XEH2OANSNfZWP193XZ1ol5+973fmKNZlKhK3U8NvPb/+1Ae+97D1Z+Se6LkvzwomF5D8Lazi7E3wBSumTxBdhElhIGoNaw8bF1du21t9vLG0cEbpEL3XHn92V82FyQDWKtDKOkDp3Q3xqNAmsRv+dKBXHiA43mDsqR15Jrce+cVh/9gZcFkeTjIBP4a7f/UggehMBleDRMzZUXiDrY9KxHvUg7Hn20DXvyL0/Zzx76jU8jTCbsyuuu0WhG16JzBQ82iCis1rLR0RF1WLGpyDG5TzbELbd8x1566WV52z332sNJFqE7is+ltkzTARsIYFEU1nCARfsLJSnm6cxMz6jDSnsmIs0IDII0Q/VUzXSb8kXctF5OyQqrcKTXpWR4koThfM+F45taX4BBPCvOQWmR69/rWlj70dExYzby6aef5dzwTEYp2iWXXqIDzz1KDxt1RdRJAoCqSCPhz1CrGDANX1GR/Oyf//yn3XH7nQFdb4gAc9BBB9p73vs+9TsQusOum5mdFEMs18mUQq84COOobxsMxxwnDBtGZXZuWpEb9yiFytDMT5sga4G4ROK+a7/egg/LFHHGR5JtoVAfmRxYd+QwY60MaJsF5IHHflz1m2qaHdaxYLWq53wc/GLVxc548EPDfSqao+bAgsVNUw6EAKkVZDI2OTlmjzz0R5ukKRwVgjINED4I6tRTT7RMh3t9lpB8EkOhnKNMWO9KGfkcxsQROlngUFeemZqwf/zjH3b7nQ/pCWNxb7zlZlk8MYkq9PXStVIVuX94eJErFtJ+RoknoIYxD8UgicqoRnifL0w/L8DN+vXrbeXKVQrTOejRIkdiS7nITFW/Rr54QP+vr1hHJ4SOh4nWwnq1ZPNTkzY9O21rr7pRJTJSiHPOP88Glixus4TwjKqpJh0sRI2QL+RKSQ8Iy7xs41QPDvj8/KyuDSOxZcsWb1ur1cMECBo9OmxuZla5JPeve04mnSSQg7nkHjWi5uSbEYQkdfGKgHsvohzWGw+4aHhYQgaEuqC4eN9tRtIUzipCCaCh6K40uLfQiMrLGUgFZWbWZqenlbsiLnDp5Vdp/TE2O6xcYcccf4wNiIo532a+8XzVNBIQfcpSNIggqgciiYpHviNnKIqyRtdde63WRg30zLhNJ2z1Bed7ZCVpHs9rOzOpNiLeaFRUfyZlIn/m7BD5lCrwsL3pIIUogbrfaO10FUhPZcNgbdoh773may1kPVAz8J7clEZNxB5QNsLkxIQWQECFKGVu+fk3C47FG59gqpmLuUHL48Hye9mgesfGIQfjcJJPefzuvFVChsmpKbXcMT0PdtE/nltnf3jyRc/VJHHqXucbZ52qh04k4DfX8sZ3NHXzOYXGW0e3Wi4LTxWqGGULF+vmYJYKBdsystmuWPtd1+LNZOzk00+xHVfsqFCPh8XCc10+bNlVPQh7hDzmaS30NrG4+QgV3Qv77BuF6qLRhQl2otlRH/ZZw95p5MoQymuCp/p/HVwPkx34wxGLoMEkvZq3zJWYElev2PnnX2a1io/M/MrXj7J93rBv8A0eDbDRoM2Nbh3VJEM+n4MLM8nbEL0VL/KNyad5VuSQk5MTPi1AFEpU9f3QdeUcDebvHCg8Fp+FJhKbkL3BgSeagxQzsmVE/160aFjPTCgw6RiIrAAwNI45wI6qE45u4+9iULy0xF7kOvEu1H5h3oEjMEYGQy55n9k5Ic3c49jYhN1wI8BbS4DboYcdZu/6D8Ta6GiiH9mbHdgLVDk4/D5NsiXPWpFcqzcTSKY3mRIwdd655wZCBAe+Zbvttbt95jOfFV4SU0D2yuT4mEvXUtJr1dWbrJp81gk/XoYEvHTtZv5kHbmvPM00AsYoU7oaqgz5fdce3apX2YQOJiCVUqnA8vDGZRY9AjAiRouQ4P1Er9ltd3v22We1+IRo/NxHS2QUIgA+8KV8L5HQgnR1d8nqR42dWMfDUqthvcoGX1BR++f/86TNFH0qu4crZq993Z526Mc+JiaJM6a8zolECRuPmySkW7J4sZeCFhyBFpCBNW2YpDAvu+JGWyj5Qn3ui5+3fV73Wh20vqDsEPNNrpP37+sbCF1CPk6D+/OSmDPLsKw8rBhKcai2jXJxkoI2YzikGAQYVarnBn3l+Of2xImItup16FYHWRzJ6lTKNj81pbEjay7/ltISNjVTDd79/ve2ZUw5zaw76wi4SJ2WNQEg8Sl+LlPD57Ou7im8UcA9QkXAIsaRkJpwm3vtyQMgEa35v2OpCnCKr8iv5fDDQIu1Sjaz571QZXkGPsRtYKDfe52Z3IixTXroyL1jGOJzlKEALESSNwBhQvxDnoih3mWnne2Vl1+W89i6dcxuv+MH6osmGrhszRrr6e/RffAsqQGr8yxwChRthV5q+MVk8gulgiKABsL1Xd32x8f/YD+6//5w/z6U+yz1L3fI+C9avNjxFgFoqGEWpN6CAin16VU7rLD5BW/KUDtoEBfUtI06Rtlr7ZhKjKaMYI/PupJ0zU+/fVqLmTBC4zro2ofHm9GAXt+I7iHYTKB6tGjRihfDHq/jegmJw+FcXuaUer21p2dAi6y2LRYGLeHAuGEzqCVLdL6WzRfmlQ9pYnqrYX944in7x/OjVmEqedpJHb293XbBxav13rOzMyK/C2TBK1a8yM2GIQTiMEUDgbVmU8c69Y03f8f+/txLlkx32P4HHmAHH/xu6+vvs54e96gYEl7L7/tA5pLrUwk1RioFQgnSn46eR+oaD2J7RJjr4Z7UtRIQ4TYVUt4UL+JhlXtfD4vcUIX+YCHLXprzdjYyE1oXG1YpFG12YtQe/MmD9qcnn1MueOA73m6f+txnFa65IcFD08XE8KtuMb1UzlmAwMBByYikQgcMz5CwlvQoKkZoh6UAACAASURBVC+SEkH/43rk+UM+SwgevRVejnyT/LEdjaj5o+agWda7feTFa1V58mjlWGO8L0aDOinhdyy38QxUMgztlLCgBKRqaDrcX+ezc5iV1kGlRXJWhq0ksPPvf3/OfvzAz6SAggG54OKLFFarYSD0BUtqKDSTKELo6ZH+tkcTC97ZQ5MDnq9ldv31N0qQn3Sq0qzbrnvsbh865FBbvGiRX7uqIR5xcT/cg6JUzUT26M3vAyVRE/9a1Ev0pQuz7dIqpU8MF3ltR2hukOe984pjxJwCmMp15W1gcFjaQXNsiNlZhTaEJdwIFgO9IW3UgBiSvHMBXJwslTZnXQ/K8ycHCbBmsLG4CBZLeWgexYox65E19noobJxicd7ynTnbsHGTPfAQM4MIq50yxvuffd43dD0YCRYAz0EzOGmvqHVwWRcKMjQAV4AvhOdszrkANjz6+B/tvvsfVqQxvHSRnXbqqaK+8X5sBJUGRM9DVBxpWK83O83PhdnxRHikeGij4oFCaU2x94ZorCehspPMPeRct26dyi4R8nedLydH+rQ/jzAUVYjh4oSKgLuAWklxEw8wsXWL/f3pv9kdd93vSoL/8i92/MknesN7kkhnQSUdWE0YEAyOG2gOoYumYzGGBwd0aPk5fFueLZ8PgwyDhSdRKae9ocu2bNkyeXEOH69nraenprVmPGcOJNEFBkM0UhH3TfuBCfQYWW/hc2mdhbl5pV4idiDVO+PyLjxfZv8op+WAhusA12ChlE8H3jKLRW7KYRgfH7UHH3zYnnn2eWu0UgK9zr/oQoGp0VBCc/Qw3eWLMKZCxRnNku+y6ZlJIcystcA45FcvXRP6fVMqWR59/LG2eNlynR2+aPTwqMCxE0Jw1aMR7gspBevhDqDiUxOC6gc1a0lEaY4VHG+X9eV3wZCkvf3zOy9poWTAg+zuZS4M9bmqjY2O2+v33VcbbOmSZWHkxBIdZh5Q9DRelHdVAw5jLJ+4En/C6kb4hYQHC+IFfTFjas5jjTKm8sLE9QxXatRsfnbGCsVZe/yPz9qLL48GnVk6+ZK2/4FvtcMOO0xIHTKX6EvR4UHIw0bFiMzMTNnwokUKUdTMQFRAaJdyZHWusGBnnEljdcv+5fX72Be+8Dnr7emVdQUQEQIMUt2ZVyTA1D02NS10WOfIueWQIsWC9RaIIhX9jIwGQEcElraFwV5bFaQfDmhUN9jmdd3jKpwObYV6n6DOoVxTSKvXhefmpm39Sy/ZFWvWqmtqaOliu+iSS7xnNXhcnDYGLl63No8+wxs3+OyB3h5dGznm1hFyYZPR5sACsoEroBtNWI3UC903ArDKJeWwXsP3ZnCF0t09WnvYSbGOT2TE+5B78j0+FwPGSBNQaLI+RNWef/55HUZVPIJUjdaX0D6R1IHGEHPgqDDgxeLEB7w5DqBaKdmG9evUPLFhEyyxhO3xmtfYV486UjVxDDPPyidUeHSj/aJ2vZR1hjY79gRccgTvuL+nnnzSHv39Y1p9bB4O7+TTT9VQcVoNcXC0xHqjjosvSISePxs1vQfeevkOy329lf54aZCcXcYyGCcL9EvO0sycI+g4ocTd153WciZMTioKkCLwZIRBLKZD1ynp5bJBPY91hDDX0eVNBrS4gSTyPbwNYWtot+vu69Wh4X1HxyfaKhiUYQiZgMyxfj29PbJWqO17aapm83MTesB33/ubdkkEz8WDP/e8sx1NTPiB4XdYJEI1RlosX7bMNm7aJMALhQi+6MFkqgB/0lj99NPP6KDv+/rX+USDLMp83TY3O6frrahTo0fhEfTHWAYiJ+MACGCq1rVhooavuocqVX2PA+8lrj43dIEhFi09axQNnyPOHh6367ihruu58fajM32TRaQREGdkdL2dc/aFyqcGh4bs4osusmTG5yU5m6elzc51xQYB9cuqVu2gGpxh8AeBlJq106VNRWkHz8i6cj/i0Qq0c7I94anWX3IwKRkCn0CfkaFns4k1FFBrDvusWuW8g4fmj5WrVskQ4+mXLl2qw6Mp8Gzmri5J0PL+XpGAI0AImbGZkJ+yRgpLg+wMnHPC6S2b19uN199ko+Mzlkhl7OD3HGyHfvRQa9B2SQlIE/e2TWpk34lKSQoHSYTcWuW9ps3NzOi6rrvmW5JaUqkrmbQTTjzB+iBTwGnPgrJ7js6e4F5UbQpG2IFCJvwBotV0b6Nbt8pB8Jooy6soJCDnRDviXTcaqm+zfomf3HZhi2Qez4GahLOjGCkYpu9Rv2V8paBqs6VLlkpAm79X6VlVztohDwOXVA3QeLS5eW3KVTvvpA8Tb7fpJQJCy9l5FDOcUCA9KknB+phFrCULB3+22Sjb9+96yCamPETnogFaPvXJTyjsmZqdbOfXbChH/5LqDIphFtgWjfcMOKZvk02KMr7LdHpLIA/He3H53S73sl09CsM4sPCvuW5a77zX1GF8BmMBiBFCDQzQ5gVwBed2Wn+Xoh8i2v39MkwAMOqL1ZDqzYoKVNjaLjzmgQlIUwdbrBNvk+l0rnGYsEhIXuf6ynbiCSfrcLEZ1q5lHMm2nmoZHTMBdzFiYB0kM9rtE+5A7oiGqNFiMCmXsN4ukOdi9BxoSmSvrntV9FMOD9dDvsyBJ58FB/EWNG86YJPyPKge8EyEnNar+j4HkfQrln2oZvh11drlJF27DrDLFMWUjIOe0cR5fx4R6FODA9GeiB5NO/HkkzTzN9PRYUcdeaTttNNO1tPX3R4Y7kqOrrAiyaTApKKGzhfrRUhOjXfzpk1215136TPpu013dtipp51m3QFJFkmkUhZar30TniPfJ3Xk2jXcjH+Des95rZ9zgKFiD3leDUCFk4K1GAbOC/Nwud3EA3dcJsojJxpuKDeAu0cWJOorp3KO+gmc0OCshHR1N27a0EZVyXFiWURsF3ltzyPwOIrnO+kzdI1eNTGEw0CeGRHJUpEDX7Mli4Zt84YRm5vdauOTs3bvvT9tP5xyuWp7772nHfaxw6ze9HoX/7FZCMuY4aoQE5YLigK1mnIxQDVm4fJvroNNBljGgWKxObBYOsIn1mNqhnqnayBJlLVWdyudzcmy4528tIO0aFZIdjx05Hnx4OKxly9f7p0mvB8Qf6BJ4pkIaeOsIG0+SeU43zcizK7cEL2ue1yMppfEvM3x0ssusWee/psNDw3bBRdeoNEVPDM3TOT/EPKZ7+O90GwqNjk/5PPTGTSavEykdchkbNPGTWp/5N7F2ir7xDoaBRSoi+hPf+yCDCoblmdPuqJul1Dj5hoAHbkeqJSF+TmRX1DHEPIaJkIQwRA5DQ8NCXhcvwH5UydOyFtlMup5Rs2T0JW1wuMT9vLzKOYAAozXQ9HigQcfsod+9ogM2qXf/KbLBNHvHO5ftfgwHV5chihC13R2mdawUbPpiUn79a9/bU//9W86H6z7hz9+qO3z2n3UZonDmhifCCG+r4sojxIYNI8GUQOhsSaodWjPMsKFXJq6c9DOis8+8ptFxAjMN13T3TevbmGtWCQW2vOJpoYUUfei5zXWkLiQqMHEQYSooIG+hK+0e6E5FVrAfMM0BSpA8BfPMnRBKLw2J4uzkbwe6nImWFAWESs0PTlhhblZK5Xm7bbb7rZKVfibVSo+OOsb3zhFdDwOaxQJw5qh37NkyVJHYTmkUTS7s9PDopBfOs3QD4NvXJ8WoMHeoS2O16vUoc4npEUyolYuFLGq3eoBFlraiSbTVtt9993VZM3G5UHwXhxOQs04yYADDW1TTRvULSs++TxeBwupxoXwwD1UJix1EXGiCnFnw5BoQDmMAtfOPbMx5a3D+BR+l++DTQCm0c5HLZV1Fxm/XcpquTHNuNfAC3JPIKWkHfybe6F5RCWJhBNhAFjEpAp1fg4kkQLrRkjLwfJIzCVvMBpEVj4LykeaqM85iBQqrcFwpJl052QYPoP8j+hN0R1zkZnDCzc6TLHHywoQE6vLa+UxR/aupAFhHOL6Jj2i9CgO0NEb1ON+EFspUHxZ73Jx3sZHJ+y7tzDNsKa1xSmccc5ZTv1U77VfZ+TCtWceg8oXCsr52UfqE9cUBFck4SC7Z3eBAHJ9DjYRC5x+rivyHhwHSVjiobvWtBgx6Vxkkmum0TWtkWhaZ65blpzFcGU/V8b3oUyIwvnsl7gQ0VuACBLqxFY9vPHM9LQsBt6GUDbb6eUUwh82EhcDOIQV5RB70/SCWtnoQnns8T/ZY394UkbEZ+Sm7MijjrDBoX4hdlh5HpZ6cxeg5rkFhjiBtYttW5EYTwjiuV9TVpVwn993BL03jNx0obFYp4RiSU9qXz96TS3lwrvtsbcOHR5WZZX+Pv2dz8SzsSasnTwmn1XzLpdVK1c6zTJwwHmAnuN67qoHRT4emGF8H91o7pPnAT4FRsD6z0xPel4ZIifPxXXc9Z6RfgrggVHEuCl/DZJDft39ogyKg02ZLvT9ToyPO5NIw5l9jIlyZJWTvJbKs2PzQaLh/VkDMaVk/NEYg0SQtgWV6FwelYMbc9Kx0VE5Dg6gpjdQmhTYWdckO3jU3DMeSyIMoP5SHWFmL9ex4OXHUGbhPRj+xvvEBhb2AmBoVJFgrahJO4EIMNJJ/eyL2C+LjpYbcP6vZi88/7L94Pt3qwIDR/6d//7vUgrxBhQOPVx+LyG5fDBytB5NxsgEOi1ALfsUI8nzi62ArHPkLHjakdbBxYjLS4f2V3ETCJVFPVOZxiVDlDMglVEs29DwYhvoHxRQ5cBEXhuG36EkRElk8eJFNiutWQcmWGSsI9aHkEYxOpZNbW8UkskvPPTBU+G1hUiHkYtxRg5Op1YuStFw3boNdv0Nt/iUd7G8Grb33rvbRz7yIb2/K/y5BUces1Aq6SG47AfKBt7xoQNLaBg6PVgMrtfRPY82+LtI5gAUoJa8V2fegZaBfk2B33XX3RQ2Tk3PCQySqBh0R4TGOjoEtmGQeChqN6tV1UWjqXP5vELNZ/72jHKZAw84UPegUDp4WylKkJMuLOi9d9xhB3l6CWnLmHhxHw9EM3zMg2K5iAcvFYlgnOJ98dxceSSmF5R+fKbt1PSEDrBqp8H7gETHLi5ycn4WW+AmJpiRO+RhNyywUKfGQzt1Mi0j6sQJBqF7PzHOAQQboIe1IqfdsGGD6I6sNXk/e2l+jqnvPhGANaDUFBsTiB4wPvGQz8/OKn9nXQX8BPJDYX7WwUPCZnAJOtF6eqwz12VbtgC+dqiZgc/j4PBzR++JLd248FVr1tTNdc7Z51kuS9NMwk77xhmWD2NGNGm+XlW6QN6q2Ukq73hzSCz7EYGgPY3zIv/n/tgPrFVspMfAqhRJpBRok3HvRr584kffu6yl0EXuOKML5hdgTnnu0KlGcw+38AqxgIzndC4mm4nQNr4P1mjRcCjF0PkfSNKx3snDQic5ItSEztyItxB6Us8NYZHYaAAuszMT9thjf7Bnnn4xdNI0RXE85fQTdYB4LxElFD7lrVh2Jg8v5nuIgvHwo1wOOTq1Xg8LfTQGm4tQ0nMl18OKXi+WTJRnZbPW09tnS5cst3Taa71bR0asp5/m7U5xlMmXyWy4Hx18wLLpGUH66vrIeWSAl1g0vEQlBUJRSQBpyIELsRNBM+aRtePhY4Q44MuXLW+XimZmp2XdOS3IikbVB5rGly1dai+++FJIKZhQx3QDrw1ivHRdMzNyy0ReAuXI18TbriospguM73GIQUmdUFO3gaFh27R5cyj7lLUPCGPj3CCfUuDaWy6iwExbryQAYIk1lUqqbs+9EplheOMeoPWPgyDEP5AyOEQYNcJhSRmFEk4k4uAE5DWpPde2TUXwkR5uuB3xzqkzCU8moCkSPJQmecSDSotmBYEnbBedUY3AmOy7776qj8f97Q0S6GA5b53rJudXX3Ag17A/XEklODmGdisF9W4wIpioxhFHjjhD0NMYnAlGIfGTO9fo4HJx3d1O78NS7LXn3vb8Cy/oge6wYpVYSngvXudzQJFc8Q6N+MEsLl/Qvcjv1LIU3o/F4CZk9aQ36zqxWCfek4VAw9fbmpyxFRX7CbXGx7bahvXr7ft3/lAaQlEB4evHHBXC4G7p82DRmE5OO5rCRw3faijnJcSL4SgbSXB+AHxY8CgSzsPn2tuatlGdMqh3gE4K/at5SEoIjbUXEIaIdtWjDv6LFpjPldxL0eVNRbHLddjmzVukErF8xY7aLNpMKEKE+jDX5F7B0Wz+zXpxSLhHDgossfiFCke0ypk0RsjRejYGUYd714ZyWIw1hjmG2Zo+MDCgtIEDTJjHsxDxXjUNJgV4OZDfLWqcqOsBA0Byb3wW6ChGgGtWjZRDgAcNhA48KgPbuA+tSSibOTjjmtwcYkTiXL+Mg+sbXDgAZSd1yczLK0rOt97QgQc3wdBzTzDhRIhI+GxaB5kQ6+/TKBLXE4tSMj6GlahQTkpcdMLcbc0RGB7Wjb0TcQOF0YFJxnPaHvCKZdLI6WfdYq3Pwc1SEJh3iSYdSPjQ0qqecVVNgW7cs5f0MEhCzR+860qhyiwKibv3vjKR28EPFp2DouFJRW9aj83vxP3KS4JiIIuANaSlTAJe0tXJtlvwonypfr/sdVEOKEgvB3ZoyBuL8XYuadKlG2GTzk5PaF7tj3/0sG3ZPBbqmGY777arfeLwwxXaU0cjFOfArVy5wjZsWK9Nz6FsAzZBYDqCZzzVqE9E2KoNWSyqiM5hZD0wHJLHIT+kuVoHOWGLFy1ViyH5Oxt+enZGeTqenPVkU4Im8wBZDyHdDdMDIb9y8GdE2lE77bqL6nkCVBLu1UFcIyuJa8IgRuSe94ujKXffbTd75dVX9bO48dXAX3HJVw4qa07aIo5w1TefRlqG8TNCzK0lMgThN0Z03br1Xr5iHAeT6oLgQQxdKzUIFA44Ue7ivdjYTmllH/kAa/YQeABGZK+99lLoSu1206bNttPOOwmEZG3Gx0Z10GNr5NLFi9spSFdPj6IRIhUiQYnei/bqbYkC7wK6z3uLRgn9NnQPRa9KAz7eGULN7KzvUT+8pAwdGvki2iRRaMajnGiQKOdg/FlDdSjh7cVDQD+cUlVJRhtjvXnzqK1cuTJQOSHpIEAxrOuNnykuROhVdnEAxoQ6YwyHE3W7uGfSCowv16gJgb+8/4YW4QCHgxonb4Rbh7/sOkD9No/anEYzFGzVyh1tdsZnp9CRwYIhrk1xmvchNCMEpMYWSQexw2Nqerpd3iCfYXH4fTY+D165cbeTGTAQgDx4CGiKauFutmzdulftttvucBCnRY9qhx1/8klqII+80wjD8x4Io0dubkQ9IwiBd+MhRBTVhejo/3UpUg1xDjNq2HRxTi6bVSGX6tg+uY3rQL9Xqn/kcINDAmswALxGiGc2o8OD1+JgIYvD/XPoXrvPaxXV8FpFMEGtYnJqQvcVw2hCcA4HXVQ8bCw4+S/q+9G74X0U7klQzdVFuKb43soP83ldM3+PKUZPb5cT+pFuEartSK84y4FPrWpCt0/Ac8wjpDZdcNgn9Yzo2WXTxUPFvbJxd911dxuiHFepSO+K+q16W2HepQEG5wOg6e2RFP4j7ZG1IzReuWKlHAHvzT6VMlGYmAgOgdGMaDH/pv6u2VdxhCXRkLrbnCQSw1KtF+iwaKeek1Ka4nDJmAZhAO4PcIn8Wg6ICEo9x3hoz42JbMi11WJIWhiINxxMqix8eQTgiDZRCgdWbYQouYSxrDHXJvVRjblU0rlQBPXgXWs17JEfMmaDw0bdjgiSjckCLlqyRHmbtGeDcgULNzDg4SgL19MFAr0tN+OwKZfr7DSQSQ1SCiUPLG5nR05yJ5ETDMghS5JMS5+KjQ4QRrsgpG7lK3i+uXm77rrrbXYWhUGsedIOPfzjEvCW6DYHIoxu8PCfMNbHo/BweN+h4WFZbLeqHpoJYg9av5QuhCAX5uW9o6aUPGYYQA1pgXo03hgQig0/NDiszxCPWTNnMj5oOekcWWp47Y3AxMICD6JPv0+3kbScQyfPyJYtHq6LMeRDwvldlRSE+Pq/QUoxMG394qBqyIPm9zTLdnBQFhsSjUJfGSMvufAesSTV1+dT5CIUHRlw7A1KGD5Hx6fIybsDGs3O2dDwkM3NOrWU9+rp7fayYhN5Xu8K4lDw+0QNdOzgtdk7pA2sobqOJNnje5D1YCPLcBRLEmEgyuAZq2MLKSBCaqiFAQvBAPMzyCGUsYh+hhYt0s+5T/SkWb84PsSBwKbjECE9QpdK3lsaXdt0sajju2SS66ppRE44fHymIkzhDN4pxl5irSgDqsOuCX3WAau4jvw75tMKuSW4j8P0hvnwIByFl0H3MTgY5sRDP7i6hfWQNEkYzSE91xQ1NBdmLgdVR8KJHMoSaBgpHNqmESw1Wak0kB/5IKyYL0dPR/4QifiIzmFR2ORYEc89E6Ii8n3AF7yTwnb6GFWg9+6O9es22g033KiDy3Xstuce9qFDPqJDyesxJEIc1e/bLdYLv4vnhfmF5cMo4AWwum4pPWRSGCMFyW41PwvoYWg2k+rVweG9sRGaj3kb90hfaewI0XCpICbg1txRXB7qDkxKn5wUQo4n5GHKC4f6Kd7HqY88yEIbrYWUwOt5ba1GiOraw2xijMhee+8VaIJ0L3W258KqZS6Q3rlu5U9C3D2EjnnqwoJ3VLHhhgcHReoXaJn0/JTckL9v2rxJhwKjBm7B8xobnQhlvLyaNYi4IjhFXVec5Q5+5iAi98hhxejwM0UGAJzq06WcBxMqKfaW5GOQPgpD1+ANq8QVOMbq2qrVbXxivL1vqFZgOGhIUCkmcAqkpIEqxbR3v3H/S5a6QDkHgrlUQoMVBi+0CUYQhiKRBWejkmkcQK7JGa61jcHnekhz+LmrdlAtIAXyPNq7rIhgQZgH5ElVsgyCfP5zb1mNgC5nkjIlLlZ740d3rRWtQ+1wuS7beeedVfoZWjSsXIcL2mGH5QGE8lYpYnh1uaBYqLEPxOqeF7CAeEM+VCFVyXMCHfSG10yxtj5P1DWN8N5sNDYNrB/EswA7IDJQVuGiG1JzNL0nr6c7o1Bgoh+AQtbO+MYZIrqLtSUVDpBP71DR4jFZjsgAiRwAjyCu7rQ838hCtfPdCpVFZEDnCKUHmrYVevqBEmAQh35r4rlHJhIfQENYAu2ICvjDVWjOjJsGEj3eVifBsKAjrNqpwAlv0GdTC6lX3ZgGBxcOJ8Tj/nzQ1oz+zfswo5XrwZsJIBGxH86413H5TIgo5HYoNsS8LZZ9eE3cILxvDKnVgkcXF/cS7hFjEUE/nAI1WIwk1xvzY1InDoL6o1MeNRBOUm9n40oNEo9a8vk/UeKHtcX78W/xAIICKN+X5GqvixJiANmv/eIf0KGVs+npMBKF0SYFat2wAEuaOhDJPSDYqslLnZS+VkaXIL/TbHPlNYw9MLCoHEiONVQSeD93DC6JxLPCeVHFYE3c+Xj/bDrp2loe+XjXlzqFqLA0mzJSNLrwjIXgy3i7cCLVEkWPqFVmaOlzuVmBjkEuKvHLB2+R4A6bhXsBIMITkRuwkVhIwjLfbJ1SAwC5w7tJTKtUbBPzuSlp4LYSYhXFRgNyMg5k9KocRAe1PJ/i4rE6nrT78CbAEfIVvg/ZgfIU3tNDu5r97OGf22//91HrQHIllbArrrxKVpmNKzkSych4aB05tHgnrCpGBoOiujGjKygvhEK3y6Z6mYTP8oVPKa9nLbztzj0714HCh4d4zmwSQ4YGAwmm+b1E7xb7TGMvLNeJ9Wajq1QRuLh4FvIcrsU3LTK3PodJXNhSSd4KY8drXQYXxpnTL32WLlGE58saZyn03NUjMURisqWZBtEVpIjmJEbA+hMBqbc1tEy64FnSmXIqw3h+jXAbeSnXHUdv8nPqvoTD3mTviv+xOYBoTTKooUnC8zwP+1U7DyguOTTeFnIPa+NtkhhJclTPodk33BBRCOg6ObaDe3QU1WS8aN8B5+AzyIcxBtKRAmkuV6T0GLEWFhjPiuHmnoeGFjkmQVQSJivKgIeZPy5BhFekf91VXSI4mWx5muYgYsL7xoOqpXdlIcjrdWM8qWYFB/4An+FVAxp0vOEj7jHuT/nxQ/ddL7E4z0e7xOkdGxu3WsOJ2yIwQE0MdDo+Tq9PJsRo0thCrAxhRo55sj4NnA3FwWEB8b54Bw4zG4mDy8YUZznr8iLcdERteS/4qBw0DozXZZ0YEnPVjRs326233i7k9JjjjrVddtlVjeNC5BAOr1fbmyl2qAA++ThFZ1nxYGP5ieuIvN/22Azau4LeMg8ecA1LiYohm5V71EYMetLx4Ea1CZVUAuvMx3e4mrD3ETPn1g0J60kTOgc41lEVSqK0wcMLYlAYMgwe+RiHjlyIPx008zICmxEPhFHU7FhULTTp3SsHkSnkNUyPZvh81oH1xVizB+L0PDWHMMAKemAq6XOLNMmgU5I2KtWNjyvSYLOxyblXZxOlbMuWrerUIvrBA0stRU0DaJI5zZAv1oTDzwaPVY5i2BdqGYRFFsp9tMPhXFTTDFPsYmTDtXmNtyED5IJ0/t5DADtoVhtig56i8bkcGtZIrZkBp2GfsK54eYXqQfVF7LpZF4Gjvc6li51Drbp0ULFs1pqqKAiwQygiGHAZIZyPKMNet5ZHDdROno83y4Qh5DRjhDWKfdPKoX96zzWt6HUAZXbccUcb2Tqi0JTNIIQxlWz3XjLyA2CGDqKF4pysOUAPelIuPpYSUBU5n4wSwUqSH/T2+CK0lQdCH6iG+DYa2qSEyVE931vtAHdQcHBBMy92t5x9AxId6m5sLLV0wX2t1qT4wKaK6vn8HpswCrv7FDQPPWMdWy1dMLNc9E/DpllUQhgOY+Qts/h4bTa99KBD0ZwSmvjWGtTkuk78G29AOAuiypsARsVGc1BJDAgglk809IZuNj2bAiPjh5v8qEMgDcCLG9WGjElku4iGlAAABCRJREFUHLkAuAOCfPEMYo/00CDtmgsqW6E7heFRvbzF5s+rrEGP7Z577hk4z82gPwUN1u9TG0rDnV1vC8EC38hzWicOBJES3lLtckQIGRc6wGPCGHIUviBjHIEZ1p/35plyT55z+8wmx1JI0SDZZJ1LHTqzWF/RalvNNjEEZxD5zUSJpD7kwp6COKkldhdFAAjsAqOAB6fCwXrwGsqjXBdeE2A1aoJTHpXWVRgMx30IeAq4DYeUZxpZXdS1Fa1pjlVZxoQoTPsj7EsYdZLMRaww39XGROJ0DHCMOOlCketvH/quDi5vitQpC7t1ZKs2VqzR0sdIvsfDQrGdiyT/heaIM1CPJ8RtwBRCX+b3dNMSZ2pWANRyDm5SHov3jaJx5DtsClfLiKJrPkSMDaiQubAgYbeIytH4oOFJ2w2X8gHEAC/T4X2cYeJe3bVs1RQQCtqE+NLUCg8yymCqplz0MDpuEq6L0hSHlUNMjiTygggGSK24hCgbS/U2Sb26zjSGI67X0mXL9H1J0kr42r0NuIAMAZpcMnquWQyAETm/fJ+p6q5i6WU0hY9hDWJrIjZE94JiBV40IK4uyObPis/HoLjXHNc6iElWWNDrBdIlgkZX8BARVCRS4Nrd27nqSYyEmNTI+4JLKH+UtIxPvZDHWzTsQGMwyBHg4/f5OWGyWFuBcBCVDsWTDmJ/3D+godD08F4YONoo8fQu8ufKGbyXUsCQa1ZDjdm7pHwNJRUj3r3rb0e+tOeSTq4gxdH0yNCdBHYgrAE1yaCGKU4yfduhm4jzQmUF58L94d2JcjylcoFAOZogX4tmG/tAEj9MhdBEDAeAo5H2PdzlQnaP/eKOFofHSxcuw8ILyJvk7eBapn1GEMVyFCAJpTX/pVbWJlfTr3RnAy+YDRAI77CMsHxCfFM+uJeNF9viVOLo7fG2qqSDEIAFHAoWVaADjQ1dPdoIKpHUnZIWPRNWnwdFQo/VxJjMzdH0H8XcHBRjcxNe6nfDOA8PXbzkozpynkZ6R1Mlxr7dRAMvo3iow/vBPeazI9UzDiMTN3e7vC0CRmIJBfqjxAoS8KN9GBjvx4Fg8xEGUq/F8OEJvdifkPdQTTWQBoRkS8PJSxO8P/VRwMRRGq41+DuntVdOzGiZMJOHDeKAYU20RaIdZzT55uKwSQo1oL9+nWnV2+O+KFeK8q5qpaTPFK1r5u+EEFe17c5uB4OIiOgiChK6sfwTh8Lx3jxD1/XyWbWUsYg08Oisgat3NCSBxHvHvJjXy6BovCtRlbf04RBE+glD0/g7835cAgc8Jsw9qjnlF1AxVkD4GSArnpUDRB0XY6TSHNTgJFxjIifmCnmDCsqP8fBHYJFnuXLFCj+ImYwOL85DVMjQiKN6MEO0Z+eUQjr0FWq3lZKrcbAuoRWQn/1fbh9VCp+xIjgAAAAASUVORK5CYII=">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -368,7 +359,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1034" name="AutoShape 10" descr="data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAALsAAAC7CAYAAAA9kO9qAAAgAElEQVR4Xu19B5icVfn9mV52tvf0CuGvohQVRaXLD0QIvUiR0IuAdFCpUkWagPQiTXoNUgKIoCKdkE4KNb1ttu+0/3Peb85wWaMmu5uwmczwLJOZ+crM95373vOet1xfNpvNovgoXoH14Ar4imBfD+5y8SfaFSiCvQiE9eYKFMG+3tzq4g8tgr2IgfXmChTBvhL3fOUeexb8798fvn9769/fWTmess6GfuRe8BSreoD1BqZ980OLYF/JdVyZPrUyoBsmV4r/VRW4fN7+PsDnKyK8byD9n4+y3oN9pbDMrJoFN6z7u22bBfzI/NsVX/kRCXC/t23RsK9prK+faszKQgvue1lfhqbWu/hm5r1/Z7M+xwJn7V2fmWYPynYM+6f3CV/wLbPavi+Ok7HtsvD5SV68IwT8ftuf//YXrfwaAX5BWvYvAXclnISf+/2eRTUMAkin0w6dSHvARdYDKgFLIGYyBtD8ILBNMjkc+5BKpezPn8ki2dWFVDqDTCaDdDqFjM0WHsjDkShC4RDiJaVAIESkAwEfUW6DpEho1gjWC8GyE0BfwCPryyJFcBI2BCcB66HTwJruSqKjvQOdbe3oam9HqrMDXZ0EZsre7+rsRLqtFV0dHUgmk/aXSiaR7uhAW2urgbmjo8MGR4Z/qTQymTSSXQR60kAdCvgRCAQQCgZtcHiDIGnvhSMRBINB+H1+hEsSGDBsFAaOHI7hG22ESGUZMgE/gj4SoaxHcLI+ZPx5srNmULCeHHWdt+zZLPmxL0cXgAzS6MxkEMoCgXQaqdYWfDxrFqZ+8AE+njUbyxYsRLoziRD8KI3FEA4EDIzhcMiOEw4H4c+mzb6GQiH4CVy/H5lkysAdDHE7byag1dcfvwBtNwdCMBBAR2enDTJuzwHEcyRTKRsA3C4SiSAQCiHrCyAUi2POwkXY7ecHY/Sm30IoEkVnNo2IPwhf1odUzvAXLX7vRmUBgD2LDJkGHUNfFtl0Epm2Vnwy/UO8+9o/MH/OR/ClkiiPxRGPxswSk5KQN7e3tiGbSiMSDtv+gYAfWZ8PndkuA7HoDq07wc7XpCUG/hw9IogD/oBRfH5GIHNQfEGlfEaZkqkkurq67H1Z9nQmZRY+GosjUVOD5ekubPitTfD9n/4UkfIyA3og6zfLbrS/d/d6vd97nQa7AJXOAS2QzSDZtBxP33kHJr/1DjYaOgLo7ERXW6tRlNaONgSCQaMS6WwGTcuaEAgEUZIo8ZiyD0il0mbN/YGAWW/j6YbkLMLhMDo7Ow2wpCR8EMh8TUtNq85tu1t9fs4BYw5obpBwf3J5EhYOkkgsjpqBjUhU1yI6dDi23nUXIBTxqIyBPecrrPeQ7fkFWLfBTqePAKVlTyWB5hb8+fo/4pP338eQxgFoWbYMHW1tyKSzCISC6EqnEAoFzSoT0AQucUwQ01oT4LTUBL5pKTlQE4yZdMYALuCS4hDYZulzwDcnV85u7p5wGx7fBk42a8enZbdZIpuB3+9D1o7tRygSxpDhI7CkM4Oxxx+Nktp6ex9+Osre4Co+en4FCgLstOzoSmLyy6/gvquuwYiGRqRTKbS3t8MX9MMXCBhV6ero8pzKdMZUlDD5dKoNUdKbdMo4OwdDV9pTa2ipjbf7vYFBUPPfoji87KQmBDMBzPOZT5mjO9xW+3MfHkOzAUGfphMaCCFLXyDoNz5fmkhgwKARWBAK4JBTfolsMAD4M/D7gj2/y8U97Qqs02A3K5qTtn0tzbjq1FPR/NmnqC6vRDqdMepAxzMcoeUOoKOj05QTD4xZxOMxj2dnskhn6JSStwft39xGdIRA9iTEtAGez/wjkAVegl5W3maCHP3RADHeTlWHgy3jBZ14Dp/fm0c0MEpKStDY2IhW+LHVgQegdswGCNAf8QeKpL2Xg7YgwM5rsGTmLPzmsHEYWFaCWCSe58a0ugSl6IfASiubSCTyTmhbW5tZbH4uoAqUBDs/M4pD6sKBkEohGo3aey4n57m0nzsTcD+Bnd+X/3bPxX9zm0SiBJWVFRg4egwCgwbg+7vugmzWjwAtfPHRqyuwzoOdwKOhfOPp8bjzkkswvL4awSDVFc+JJCBlgfO8OU1dvMveF/jNwueCTeLUsu78TO/lAe9szzvA9/nQ8bi9rLcCWJoR+JozgXwAzQjcJxqNIJGIY8DI0WgJBTH2sMORjcXykmev7vZ6vvM6D3YDZDKNx/54E16+9140VJbCFwiZJaRVp/WWZea9JrAU6STYTFbMOZmuyqJtCVDubxw7R1+4n94ThxdN4WecNfiaf6I+whlfC+zuIBGNiUbCRq8qGhuRDkXwg7Fj0fC1jRAMR4rSYy8H67oP9kzWtPN7Lvs9Xn/0UQyoq0SA6gcDS6GQgT0Wi9m/XZ2btMU4PwNPjlU2Hp3LTREdcT8X1ZESo+vP1zy+9pUyI04vYLvyI7eR46sBFPD5EI9HUV5fi4aBQ7GgM4n9TjsZwUgR7L3EegE4qGnmpqRx12WX4x+PPYHGilL4/F6UkiCnw8c/WmKF/wl8KieiLrL0fF90xbXsAjZnCllrUR6+dqmN65jq+AK4tHYdQ36AAk1yiCPxGMrLy/H1r2+M92bNwc/OPgNVAwYUHdReon2dt+xUXZDpwv1XX4sJ996PobU1CIUillRF8MbjcfuzqGVOQiS4ZOXlYMrycoCIqwvwepbVFnXha/5bSo2suWYHPUuBEegViNJ+7vH5WTQeN+4+ZsMxSEXjGPr9LfC173/fYgJfShVmukIvAbA+7b7Og50SYjbdiSduudV4++DqakSjcfhyyVhlZWXmpMphFLhlRQl60RSBTo6jOLyinnptmY05i07A0uJb2oAjS7qcXVKkVBi+1oChtRedkiMdDsdQVlWKIQMGombwULSVJbD9fvtbUhlz3pT3puDX+gTY3vzWdRLsAp+ndvB/SfzlzrvwwLXXYUB5OeIlCUsmkRpDy06LLUeVPFmOqaiFLqLoiSy9rLcGgktB3Agrz6WBJFojNUbHJMg5uPhQWoHOr1mDAzMeS6CkogTVFeUYOnI0Pmlpxp4nnIQ0Z5JgwAM7/11MB14t7BcM2F958CHccenlqEskUFlZbekAfBDoBBBzV1z5UGB3KYsrDSpKqmioVBk3cCSu7c4Iokd6z5U9ua+iqMqW5Hv8LnodCoQQCUcRLY+ivroaAwcPwbS5n+OQcy9AIB63IBTTzZiwRrAXM2ZWHe/rONi9aiBkkvjXM8/gpnMuQH1pAiWlZXYFCHA6p6QZfHZphHi0q5oIiArwCLAEo3i2S2n4HgeQBok7O4jqyLprRugufYrC5KkNfIhEoigtT6CivAwDBwzE/OXLscUBP8PwjTf20h+ZT+Njnr4H+OJj1a7AOgn2L/00SxdI4p0JL+KaU84wsMcTpQZw/RH0VDcITMmDBFdLS8uXMhgVdJIWTmAzP0aRTgFefF3URZ9rFugeoJJ/oAEmC69B5Tqw/IwDk5Ip/+rq6izvvbW6Cnsdc7RVNtn38LEwpcjaVw3m3lYFAfYMkpj55pv43XEnoSIcQqKs3JQYgltae2lpqb1Wiq50cQWARGdcTi2rK4dVVlp820CXy1+XE+o6n9xe0VPJjJo9ug8MNy2Yg5Q+BsFeVVWFxoED8eqMGTjzmqsQiJXktHzGA+wWrs79Xq+3XafBblIeA0NI4fMpk3D50ScglkqZZSdXJ0hp1flvAsd1DAk+Wm2CTxq8JEkhQjxaOjupiXJf5HTKqruzggaJnE4dh/vwfC5Pl4Kjc/I4/M784wCtrKzEiJGj8Pwb/8Lxl1yMqsGDActtL4J9dUduQYA95Uth6UezccEhR8Df2oqysgpzSmkhCXTSAsmP3Z1UWXYCmVad/FyJYwKt1BXu684O0tFdwPIY3N/NbpTM6PoJPGb3hDH5Bu4gJdiHDRuOqR99jK0OPgCjN/82fKyMkuJe7ESwypgvCLAnfSm0zZ+HC35+BLLLm8zBI9BNxovH83xdeeeysLxKoi0EIlMICELuJ2dWOS9SYaSfS5vX+6JFPIcVabPmNJk0Cy3aI2dYUVZRH5fLK/hFGsM/xgkGDhyIQCSG6AYjseVuuyJrtam5tIYii1k/wC4OnUIGnUuX4lc/PxTpuQssTZYBGAKNwKWTR9BLfpQVl4oiYAqkbm6MJEhRIDfEr/fcIJS4tzR3RVgFeAFcn7vAdzk+Qc/vTCpTXV2N4SNGYH4gg52POAIZOqk+f1FnX2WYF4iDSiudQhaZ5ib8etzhaJ39McpKE1ZiR4CRwtTX1xtoFFgiqLuSSXQ67TKUb+5GO90opwJIypQUR+f7Lm1x+bmSzJT56EqUipxqEOi4yoHnMcXda2pqsNFGG2HykoU4+OyzkA6GjLeTzBQN+6ojfp2mMZ5lp4Oagb+jHb899jgs/GAK4rEYIlHPqtM6kvfSQeW/3WILOqiSF2VhbfDkCjJk1QVSOadyWBUMcqVJl7+7aQW6JYqYKmWY77sDTLOKl9vuff+KigpsOHoDvP/5pzjivHOA0jIvhbgI9VVHeiFIj54ak0WwqwNXnnI6Zv39n1bHGYl5UVMChryXVIB8WlSBQGfmIzm75EDXISVo9dp1HEVdJFWKh8uiS2p0+bnybzQodFzNDhoAbsEHB5aCYVWVVRg6eDCmz5+Pnx5zJBo2HGNdxALFjgPrH9ite1ZnO26/8CK8++wLSJCfx6IGdP5JwlNlkhxUlckR9AoUib+LTgiQckTFyQVYXW0pK92vvhQbpSco4OQGktz8HA0anp/fl9+/orwco4YNx9JUGrUbfwNb7TGWJVHG24vGfdXxvs7TmHzP53QK91x5Jf5234OoLI0jGouazk76QsueSJTltXepMMpvF01R0bQA7QK4e82owC7a0j2dQBSGx+QM46YBd58V3HwaObsEvWvdR48ajnhZJWY1Lcfh5/wGqVCu/UdRelxltBcM2LPpFJ6+7XY8c8vtqEzErCxPnJeALylJoLS0LF9JpIINUhjxZ/6bwCNwBTqlDsjCuzRGfJvPoj0EqQpDZKVdXt7dssuJdbMpdQ6BvbSU7TUaMWDgEPxz6nSccPklCJZVIsDOBEUPdf0DO9JpTLj/fjx05bWoLi9BMOQ5ePyjIlNZWYWysvJcew0v/7y1tdXALwvPZwLezY2Rk+o1VPKKNbrnysipzEuhTr2qm92oJDIOKDfopHwdV6vnv8nhLZJaVoqa2mqMGD4Kr0+eioPOOB1Vw0fAHyyqMauM9EJwUEVj2BHsrWefw63nXICKRNTUGAWWaNkrKioN7AoKEdjqxitVxg3ni6YIyPm+MGyrkatdVdG1BoSsu2iSAk/63NXW3VwaV8ZUGgL34fFUNF47oBZDG4diflMLNh27K0ZuvpmlMRct+6rDvXBoTCqJaX//B6477SwkokHES+JmiQX4+vpGkyCVaUiwkW64kVOXS0uCFAXhdpIaxc/F12XpZY35rBlCt8JNFdB5LLcn1wdSg0sFJgI9ZyYO1vLaCgyorEdpbSNio0Zi0x1/DB8te5HGrDLaCwDsuR7/mSTmvPserv7laQimk0ZdCEK2pWCXr8GDB4PBGVdVobXmH9ME+Mft3Q4Eoi5SUrrTFUVH3SipuL72cdUc3hXlxLhZj64aI/VGEiZpDINhpRWlGDxgEBoGDUNrLI6tDzwACAeseMP9Xqt859fDDdd9sOcqkDPpJBZ8+CGuPPlUJJc3WRRVDh6tI1vKybITkASdyvNo4WWJ5UC6z24KgFuU4SoxArwwpAgpn/ONTHNVSd2VGQ0McX7lx2hgEuzl5aWorq/FkKEjsSyVxa4nnYRMyAdGA4pgX7WRWzhgz6Sw7LNPccWJJ2PFp5+hpsYLIhE4tPK1tbX2J8ohmiKtnc6qW4zt8ms3CKRIq8DN7dSlV2kBoidSdvS+jqmorbaT9Olq+Do+32MEtay8DFXVlRg6ZAQ+a1qBA848A/7yUm+FkSKXWSW0FwbYrX16Gs3z5uIPZ5yNBdNnoCrHzwl26uwNDQ0GGqkp7I3OXuySHemkSo6UoyqlRiAVzVG6gNtjRrTEtfCy7m6GpIo7rMNwrpe7m/0o4OozHoNVVpXVVaiqqkRjfT3mLW/Grscfh5pRI3K57UXArwra132w59aqyyCD9oXzceM552P6P99AbXVVvlpJYGckVX3VZeElAxJ8bpRT1rY75SBwVXcqXi2gC6ByYJUy4JYCKlClc2mwidtL0ZETy5vI711SWo6KigQaa2qRDIZQs/HXsdVee3rpvjlJdFVu+Pq8TUGBPbliOW78zXmY9PLf0FBXm29cSq7O8jb+idrImiqoRLC7ll3qiWiO+LkALMqhomtXydEAEQd3I7Iu2N0Bxfd5fll2pS/wfcvYLImjNFGC2ooq1A8diokL5uKEiy+CLxy1dtZFKvO/h/E6D3Z1yMpkUki1teLmCy7CxOeeR601S/qiWknJYHT2+L4AqeokJYQJdASitHVeRpdDi4PLGsuhdOVJApcDRM6wLLnL5zUj6DhSgjRjyBn2eslEUFZegZqKagwbPRp/mzIRx/72HJTVN8LvD3vL0NhialzDtbhwwcqgXzBg52JcmY423HbhJZg04UVUlntF1ypeZtYjHVWCXj0bu6cMUH4kAEU73EalruXVQJH1lb6+Mi3epUGaTdzqJ3dwuSkJSiPQTFRaEkMsUYqaymoMGjoUHy1djG0O3BejNtkU8DG/3QdfEez/1byv+2BnYMYHWy3Dn+rCPb+/Gu8+NR7xaNT0aSWDkcLQQRVvl8Iix1SpAnwt+kEgurKgLK9oifLbXe2+e6qBG0zSOTWgNBDcHHelF2hW4cAwyx4NI5ooRUVpOQYNHIxAWSlKNxyOH+76UyAYRZaVS9Zeg9a9aNkL07LnwJ7KpBHKpvDQdTfiHw88hDDXJ8q1z5BFp/RI/i5+S7BJa6dV5zqltuhvroe6opvi2aI8ojFu3osGiCKffBbP5/4aKHqPg0pWXb1ppPoozViOJwNLiVgUoUQJSksSGFQ3AHWDBmNOVwsOPe1UZEMRZEiZ4C1yDFPfi4/uV6BwLHs2jWA2jWfuvBt/veteZFJJoywqb6N8N2DAALPuUlMkDYqvU2t3ebpoibR1qS2uI6mIp6Kj4tnaVtRE8qPL2fWeLLsrVfKcKubgACmJRQzsJfEEGipqMXDwYLz56RycdMlFCFVUAgGump2B18mmCPaCtOwsyWPun1EJXwavPPIEnrvuZiQ72lFdU41QKIBQOIDyiioMHDTIrL0bEBJVURak0nMJMDcLkhdPujrf7y5BSlnhduLmuuDddXRtq+Poc5e/K2FNFMmaJpUmrHNCVUWlDdyPP5+PLfbbE1/bfhsEbM1uLkhWXEbyP81p67xlp77OlaBtTVFfBu88/zIev+IatK5osoW4CPZ4SRS1dQ2oq6+3Ag5lIYqmELi06GyHp9wVBZR44UgzlG8u6VFgl9UXjxdHl9bOz11ZUhZfpXpyRHUcRV1Fg3gezU58tjyZ0lKLBocCEXweyOCoC89DOFxi7TWygSxYnVp8/PsVKBywG+gzmPHPN3D3+Rejefky1NbVIBQMIBaLgFmPTAQjf3cLp13OTlC7zqK4ujsAxL0FdtEYV0kRPZGVd7V53QJZdYG9e5UU3ydX5/ta8U/KEp/ZHmTIwCF4dcokHH/5pageOAhZP5DxZREs0piVjvV1HuxZk9volnHF6BTmfjAFN591DlYsX4qq8grEouybSLA32J/aaYh3C+x8rSZJUktENxTllGPrvpZD6jqosu4aLHotvi66ooCVq/poH9EmzRikVaRR/P6cNWjdNxg5EnObVmDLfffB13/0AyvCTmezCBZXwy5csBuN8XGJyCSWzvwIN571ayyaPw/VlZWIs6VGJISamjrrH6MW1rLEqlJS5qOriLgUozuvliOqgFN3sMviS8t3HVcda2UziavFu3RLkVothkbr3lBfh5oBg5Cpq8Wuh42DLxwywBdpzMpJ3Dpt2W3RDa5dyhbt1qI/jZb5C3HdyWdg/qcfo7a8DFHmg8fjqK6usWQwyZHdwS4Lr8ajsrauVXZpjZZu756XIn7Obd2QvwYRPxe9kTMsvV3PmnUkU4q/K0imnpOVtVXYcNQYfLhwAY6+5EIESsutY3sgtxBDkbd/+QoUDth9GSCbRsfSZbjpzHMwc/IHqCktsXySULQE7L3S2NhgVT9KyeWlEHfms2ntyWR+9WnXKruWXOV8Ar+yIOWUysobDeKKxLml4bW9QK0kNPc8blGHmyfD912wcyCUV5VjxJDhmLt0Gb67zx7Y/Mc72kqB/lz1UjFfpkDBnvVnwQKOdHMrbvv1+Zj45r9QznwSdhYorbAksNraGkuXVZdegkGOIQFHq97c3JzPIhQI3WxIpf9yPzc3nsdyS/64naw59+f2GgSiJyoYccGuNGJuq6CVZgPl2vCZA6skGsXwoUNRWl+Pz7o6cfR558AfL7G2eO7+RQvvXYGCsux+ZJBubcO9F16G1195CWXRiOXIROMJ6whGuY6BJqocchZlybVIAcEubVtlewSWrLmoiUtLXCdVs4XAJulSdEiJYfIHXCdY9EURXMmWGiSqT1XXgYjfj/KKCozZeGPMWbwEY489CvUbboCA30sXUEJZEewFCvZseyeevOp6vPSXpxEL+FBXW4tIrATl5RUYMKAxv7x7d7CrwwCjqBwAStbi+1qsgO+LGmh7l8oo4inQCqySLkVRXEvu+g76vHs2pMAqsHPAWHezbBbRkhiGjxqFmtoBKB09ElvutRuCUW/9qCLYC4zG2AoUtq6SlxeS7UrhhZtuxwuPP4pQNo26ulqUJMrygRjSGAFBNEY5L6IbruYtgLu5LYq2ynqbJbZ2dL48dZE1doNKkhwJViWcaWbRTKHtXeBL2VHk15bPCYbsN7NlSF1tPUYOH4VPOlpw1Hm/QaSyxsuC9HutT+kSF5sQrOM0xh232Yy37Eo2lcbLf7oXEx58COm2ZtQ21iJRUoaqigrUN3gOqpvAJc1cagxByD85ne4AkGUluDVAxNX5XUQ/FCUVb3eDSuLrArkiqYrmSlcX2AVwqTtKQjM6lM0gFo2iKlGGoaNHosWXxpgtvovt9zsQ6VDIIB6gLOuH14VgPecz6zRn/3ew+5BNpfDPBx/Fs/ffj0xbMyrrqpCIJyxbsLauzhxVF+yiEZIB1VZD6QICqlKBVcMqFYdgVX92KSYujXE5uaiRrL7WdHI1fJ5XtEcA1+cagJI7swEfYuEI4qEIGhobMWzDUZizeDEOv+B8xOprCXUEGVYt9j9d9x3U/wT2tx5/Cs/eex+SLU2oqKlELBpHOfNJ6uos65HSo+iCG+AhMAl6Al5gF/AkE2qgSEnhPuoMxu9D4Avs2pfbKKNRygqPI7BL7ZETK+uu2cKdNTQATOb0AaFAEOxRRml11OhR8MXjGLP9dvjWjtvCF4ogqPU51nezvq6rMf8J7O888TT+cu99aFu2GBW1jKLGUVleiZraGstnZzGELLrALuWFIKaTKhohNYXPcixd8EmCdPVxcXlt7waaZOkJdjdVQXxeer4c6O7HVYCJ25OT008gK2eC28DGAdjoa1/HvNY2HHLO2QhXV3vL0dCpKSaHrdvS438E+5PjMeGBB7Fi0XzUNNYgHIwiUVJiEVTSGEqP3cEubi7nUzTFVVBkeXlelezRwrqLGbhKjhvUkW8gyVHOMd938+r1b5er63dyWznXbiSWKQLBSNj8kg2GjUQy7cPArb6HXQ89BP5QKF/Qsb4b94Lh7OLB2XQak5+dgBfuvx+LP/sENQ21iMVKEAwEMGjQoDzY3WimrCoBTArjluoJ7KIaeu2CXQEjN69FYNSgEvcX6AVyNy1Big/fIx3Sa5fri8bo99pnVtztRyJRioH1DRiz0dcwefHnGHfWGWgYORr+YAQ+y5lhnSrnAa+UcX1bpqYgwT5twst48c8P4LOZM9A4qAGxklLEIt6qeaQxWhyAgHHpg3rH0FK77fBkyV3e3d3xlDzYPYVA2+lzBa9k4Xls5dm4A6o7fdGM0Z3m6Ddwe9Kz6qoqjBwxArHqarTFQhjHzmHsSx8MWQ4Ra5hsxY718FGQYJ/1ymv4++NPYPbkSYiXxVFZVWNLtTCKqu4CblKXpERxaDmq4s3ctrskSdDRMZVVdxUe8WoB2lVbNLh0TjmqsvhugyWpL25wqnt01eX23JfdiwcNGISRI0dg7rLlGLnlFthl3CEIlLBVng9BNlTy+c3Cr29aZEGC/ZN/voF/PvEUpr37NkLxMGrr6pGIl9jiueobI8VDgNRiYsoxF2eXouJmKArgbi8ZN49F6QPdI6h6raCVCkWk2ZvT6fNKDBVkktLTfcBosLqONN8LR8KoLC/DwPoBGDx8BKYtmIe9jz4a39xmG6/vQMjrILa+RZpsZs2KXBbAtGZWLp3G5/96C28/+xwmv/Um/GE/6hsHoCzhLZ6rFF8pKuLM6gzGY6jyXykBLhip1IiHywGVtVVimECrz13Qu8llLujdXjJ5/yOXDqyAkwCvgaDtdD5vkPkQzTmrQ4YOR6KyGouaW7Hvqadg1De+BoSD5DGeo7se0ZmCBDvSGcybNAnvPP0Mpr/1FprbVmDAkKGorqyysjzSGEUxJQkSdC5HF8jdJDECiqB2FxkQhZBC4vJwRVa1n7IZ5fxKepQV14yigSPbI4C7lEjOrsCuWUp2i84q/RL+3kGDBqO8qhqzm5tx7NlnYtCGo5ENBgFfAAFrm2fDHuaxmm5TeAsc6D4VnGVHJoOF06fhjUefxOeTpmDe4nloGDQI9XX15pwqxdeNUoovC3AK9vAiuWkEogyiuwKyJEGBT1RE4OOzG2hSgYibEKagldQW1+HVeTQwNCu5x3cDUYqwasHgQYMHo6SsEiuQxh5HHobRm22OdJCt+bwlc3xIewvNBpMAACAASURBVFY+B/hCW85D960gwb5k9iy8+eiTWDjjQ8z66EOUVlWjvrbOdHb1aNcFkFqiKCcBqCanBL/6tktFEWUQwN1MSOWZC8xSSvjM97Qqh6y766y60VZuT64ukOs76jiufi+LrxmBdEj+g7oR0F+prahB5YBGLE534Ts7bIcd99oD/njc1lNVwpiftMk0ycJSawoW7NlMBis+/QRvPv4UFk2fgVmzZ8AfjmLo0KEGdPL2la1LKodUlpyWVqtgi87I8eSz+DYBKa4ukIkGqf2G/ALlshPYbmZld6C7M0P32UHbamoWpZFfIIqmZqv8DkyPiCcSqK6qRsOgwWjt6kJVQz222nMsNtxsU/iiUQM9nVbKk4UG9vyMW3AOajaD9vnzDezLZ8/BlCkfIJkFRjHnu6bGgkqc3mUtpYgI0LK6BL10dz2Lm8tiK2lLlkOWW/TETSZz1ROlJgjIcjg1u7gVT6I1ojlyjt2gkvZzuTsHtOiMWfugDxWJUlSVV6GuvhEVdbWYvWAefrjLLthm773hi3n9Ir1lawpArej2EwrSQeWPal+yCG8+9Dg6583HxMnvo7WtA2PGjLGVK5QuIIogsEv3lhKjHBlup84D4tECuetE8jgq8pBTKQutgJAokBu0cgNbojWiQ/pu3QeNBomOpwHgOq4qJFGrv1DQj0gogng0hnhpKWoa61HX2ICFy5rwg912xxZjdwUiYcugCTAXvsDwXlBg/0JBzaKtaRnefeBxpBYswnvTJmLZsiZsOGoU6urrTI1hpFFOowt2gtAt5JDFZAqB8l9kofmZq5QIVHrfBTr3JX+WY+n6B919BwGYx5OfoMGlCKsoi+vEKhgl7Z/nchUhzQTWNzIeR6K0FHUD6jGwbiA+WrwUu510HL7xwy3ZmwBBWzm7sOBesGBvX9GEiY88hY7P52La7BmYP38hRgwfhsGDBxmFcWmM8k9IJdx2Gsp8FHhVWSQn0eXO3Z1WvnYdTKk94tkaUHJyJYG6PFyUSA6wvocGp6vFy1cQHdIgkHWXkVaZnhzXsvJyjBo2AoFEAs0lURz9q7NRWlVjeTRFsK8TU1sW7SuWY8oTz6Llo0/w8YLPMHvWHAxsbMDIUSMtgspGSQKNQCutXfIj+z6qyJrgkEKjFAHRHjmhArQaovI8rnau8/ASupxdM5IGnay/LHN3RUYzizuT6LaIs4vny1kVLZIvwO3ptEZCUeu40Dh4INp8wHb7H4DNtt0WvghX8igs615Qlv2LcZhFV8sKTH3qeQP73KXzMX36TOtwu8km3zI1hjTGVUMEXFdyVLcuAkcDQeARfXGzFOXgikZwWwFSAJW1FOik7riF1JIOXYXHPSZ/p9QcOdHKoCTd4iBVYhmPL0dVqpGOz3OGA1FESqIYMrgB5RWVyNbU4biLfgtEIlZTW0gPm30LSY3xbk4WXW0tmD7+BbR+9DGa2lswZcpULFm0yCz7sGHDrFpJtEA6NcHqKjGu3u6qHQS4q56oOxetP+kRwcX3CFY+ZFVlqcXdBXQNAM4EGkSu0kJwihIJqK6DqvOIx/OZv2PZsmWYP38+5s6diyVLluQT2XgMlRYGAzEkKkowsKEKjbX1mNPSjrNuuA5l9Q2e9i7evo4njRWkzi6wJzvbMPW5l9AyczY62prx8aefYvr0Geacfu1rX/PaPYdCBnhZRYFdVlyKifLW5ezJYhNk6q7rSnyuoyigC2ACvAaBqMLKKEP3z7q3xfjCIf9yP3hxfZ5DoOa2tPrsibNw4UIbCPxb3tJsBerVpWWobqjD583LceJvL8SAjb9pncXy6QP8l8WZvuy05lJ37LLn/dls/5Mu5QsVnGW3/o+pLsyY8DKac2Cfu2ABJk2chGSyC9/4xjesiIMWmABX8MilBAKKgCsLJ/DoNQeMLK8srEDpWnRebDmL2td1AN2op6iSrLtAr+/iyp/aVpKjLJjrkAr8Wv9VaQv2GyMhZLqSaFnWhKa2Frz/4TTsdcTh2Gjrrb3GJOwK7PMhm/UhspIV+FgE4g5g9zv3JwpUsJadlz+dTmLmX1/F8inTkEl2YeGixZg86QM0N6+wSGpjY6Pp7U1NTZYOoPC+AOGCXUB0QS1LzYuo1ewEXlkRDQTXArvWWe+7dIYZi1zike+59ESAl2qj2cUdMDqvlCHd4O7UR6uHGDDZdSDL5cZ88AWCSLGFYCSMcEUlomVliLMLcnkZYuXlCEZjXmoBTbwNAOsqa8aedbDGdPqxXFmQDiovOvupzH39Lcx76x0kO9qworkVU6dMwsKF8y0/hq2r6ahOnDgx3/Oc4BRABSY6sgq7qwuXu52rd8viyrrJksvqCnTuQOJ5+LkcVJd3uwNDAOX23Z1d97jdUwbcqC2/P/+k2NisQIga7XDoCVPds0wNA1Is8ggFkWSuTnU5ahsb0TB0KKLlFUZpOEA84HN5m/7dr6MgHVSCvSuTRtOkaZj92j/gSyXRvKIZ06dPxWeffYJojKVr1Rg8eDDee+89cyrV81yyJJ9psQVwSXmulXcVEtGJ/ybXCagusFyKomnfpTHdLaV7DHc7URwdQ7OGOzjcQcHt5KBb5zCzzn4vL8bQn4U/EEQ6nUU641GVVDaNLtYLRCJm9asaGlA2dAgqa2sRCAWtL3zWBk3/1OgLyrLnaQHrStMZLPvkI0x57kXEO5Po7OrAlKlTsGTZEixvXoG6mloMHDAQ06ZOtZvEiCJrVIcMHAQGWqJxb3WL7oBy+Wl3NcWlMXJApa3LSov+uKqLy68Ffu4nBab74OBnHISqYOLn4uVKN3C/uzsA3UGp3+IGx0zuzGaQ8nu5+wbyVNoGgT+ZQoo+TiqNzq4UItEokrEI4tUVGLDhaIz85iZAJG5cP6Ce2f2IuBck2Hl9edPbFi3CO0+OR6K9E53JDrw/8X2sWLECcxfMN+lx5IiRmDVzJuYtXIChQ4Zg9KjRqKvyMiLDMY++uLRC4OjuiIq2rMyqCqguveB7mhX0vmiMzqH3RTlczLh0SUAWiPOqQ45auJTHbeSkwScfQM9eslkKSa4Wnlv4zCw9jT2LV1J8374lF2+yUo9EVQWyZaXYeNttUDVyFLK2RGU/QnnuqxQu2JFFqqkJbzz2BOKtHWhvb8HkKVOwYO48A3uirBRDhgxBKp3GhzNmYPjw4RjCip5EqfF29mDRku+8VgKj2+2LgFG4XwNAYJMz60YyNQgFIllf17J2pzI8niy5gkwu99b5NMtoxuAg8ax9Bhnrgem11HNnKneQKvnNC6B12hqyytzUwJQjHgpGDPB8XcZOwpEwghXlqNpoDIZ+59v8oF86qgUNdrS34a2nxiO0dAW6Otswe/ZszP5wJubOm4dQNIya+npMnTYVjfUN1ta6JBZHIubxd1p2cnnp6KINinyujCO7qbcaIOLGrtUX3ZLjq3QAWWwFrOSUasDk5bOck9p90MjZVbsPRUz57DZxYnRVg1eDRZTFBkgmjYA5qR5/zye8Wbkeu4uRQhHQfoQisOZT0UQZyoYNw6itfmjt9/pTbaurehWczm4Ay2bg6+zABxNeROrzBUh2tGLBvAWYMW0aPvvsM7R3dSFWVoL3P5iIhpo6DB40CBXlFQjxBoZCKK0oz7fJExWhMmNWn+2icxmMrmIiysDzu9VLGgQCI7fjMVRAIqmQ+5FGaCApr0YWWIDUsfls6grD4Lkek7yxSjXWQHPTjnlsUSOBWDPUF7MUfRVvePIzfU8CnM5nKpkytSYai8EXySDBLsLl1YgPHIwR2/4IPr7fjwq5Xem3IMFuwMsk8dnb72D+e5PgSyaxaPFCTJ00GZ988gkWL12KYCSETz/9DMMGD7E8d16UaDhilp3OF8GtthsEDF8rFUBW2XPgPHogMLuOn2vZZbnF2QkkRWddCVNUhEAWAAV8VwFSuq8sub4T9+F22t9VfDSQ+J7ydhT8cilTJus5p9w+FAojFAoinWLnAo+6hUNR6wsfjPlRGStBIl6GSEMDhmy1JbIltOz9K68mPysWXm4MTFHIZpJWqTT7b68j09KC5tZmfPDBRMyZMwcff/yxgXfp0qUYNmSoOazi1FI3SGG4DQu0ZcEJdgGJz9xGOef8d3eHUYAUJRHgxfG1vVuALdCJy7sRUFllafikJDwGKZfr9GpAST51B4tmJff48jHycmRuFUIdR9ZddI7fl5Y9Vh5HebQEiZJyRBobMHTrHyAbjSLQz5qoFjTYufAtwd61aDGmTvgrfMua0dq+Au99MBEffvih8Xda7daWFpMgGU11ubGme02BcgoFdC2vLifTtcYEiEDmqikCuMvf5Thyez5cn4AAtaVkzNH06Ikojd7jzKBYgL6bjsl9lP/jOtOSPzUDiLe76QRycHV+Obb6flp4OJyIIRJgAlwpSocNxbAfbYks4xP9iMZ86XoXmmW3KLb14s4g1dqKSS++hPSn8y2SOmn6FEybNg1Tp041sFNKq62pzS9QIKdOyodSf2VtadFcCiPrr7I7zgKcDTQ7aEbgcTUAXJ7vgkqKiiva6fvo/C7dkZQo8Cr7UsAUp+dr+RMaJLJ08hfc3ytaIydWA1G0hs8cBObDBEOIsQc8+98PH4phW24JlMRySWPuL/nq/22/tdDAnr+sGSoJSXw08X0seut9BLo6MG3GdEyfPt3SBJQaQJ7OtniiAaIcsoZSM2hFxcdlhWXh9ZpAMZ0+F33VjEBwScoUwLvLgAKiO6uIRsgfcJ0t/VtUSDOHwOoOFPkO3c+hmULWXZZbKcqy9uL47uxka8lmYP4N89/rxozByO99D75YpF/q7AULdlPN6KMijUx7Kz5//W0s/HAGPpkzG++/+y5mzpxpbZ7j8RJ0tLVhww03zHN2trZmzgdTPaz7V8pbP8n+nUlbc1A+CGo9ZO0Ffjd/xqVAsuqytnymhUymktadi6DjcaVxSyMP5PJOxPltIHYlLUyvY/r9XBvVy1MRvQoEA/kilSBX6GAnsJxaxPNqppCT7YE9lzqQi9LyPS2SHAxx0TKfnZfX+LOlS6wtx5bbbYvhm2yCSH295QKH+2FCWEGC3RLB7JZ4PVB8mSxSHR34+O13MOW1V/HGCy+gdflyzF2yBImKSqSTSVTV1FigieJy2BdEOpfJl0p2IZ1KItnVgZb2Dhsgxu19Pm95l1yRhni6KAUBQpokoBvF8HlFGK4Tm0ynEAyH7JhfqDTs3+JlPvL7cBCEggEvhM/zJ1MI+gNIdnXZoPRZkYgPAZNEg7CBkUlbkheTs9jzyOf3WWYjO4Ax0KTkLT9Xw2ZaBCXJVCo323mR0SyLPKjCAOjo6sKiJcvw+YIFmLtkKZo7O+CLRNDSlYI/HMbdD9yPBFchDPJ7e90J+sujoKVHgj2TA7u1ZSZmuKz6imbc9rvLMW/yFLQsXoKFC5egsq4O/lgUAzYYjm9v+T28/vd/oH1pE+KdaSvj4z3r6Gq3qGJrs7c+qgWBqOPnKogEUiWTSYvXuk2y+uGAl36gASDrLqogwJuuz6Qqk/58CPi8NU+TmS6bVfgxLX5nR4fNXrLYjPrasQn2NPNngvD5aYn9tn0gzBmLyyITjVxUjMfibBCw6D8HFSlWS0szFixehDmffoJ5ixdiwbJlWLp8OZpSSfhDYQRCEUS5GFtDAyL8Tdks7n/oQVRwYTYe1+sW2V+w7hmNXApJQXL27tyWrz/56CMcfsDPMLymGjFa/BSwcMlyzG9aimvuuhXf2GwTdLZ34ONpH2L2u+9g9pSpaF68BMGuFNIdHWhpa8aK5mYvQYq6OleyyJW4idaIq/NZ4fW8tad1z+XbhMMhLxjEBCsCg8UduVbSTGIjoC1QFAx5oPRsrZeTQiuczYCzQsgfQjgURjgaseORXnSkupAN+REMRxGOxBEKx5AoLUOsNIZQNIJoaYmX+xOL2oAghWEV04qmJixbthwtzc0Y/9RT+GDKVGyzw3YYOWYMOlMpvPzqa3j9jTcQ8IeQSJRZMl2IoVZfFvfedx9q6+ttBuFX7E9gl19i/lYhOqjitu4PfXL8szjvnHPRtnQBsqQAaT8CwRAq62ox/sXnLWpqQRf2g0l3ItPegfdfeQ1vvvQK2hYvQUvzMixZvAhtzS0GUi7JaPw4SOvoURTybVphrrXKZ34uqkPQqjpKfJnUg7RCtpBgMbDTIjNHnPnuuSVn2HW3oyuJUCxi65pmqK+XlNjiaKF41GgYl3Yvra5EtKoc5eWVCMViBnZSnSyblwYD1qPdxpflowfyNpjW35ZOTmfQusIDfl1jYy6CCvz9tX/gmKOORntrG0pKEraKSSgSRGdXJ+6++27LNbJZyTql9h/L7k4xhQn23C+0deSyWWRSaVx04eV44onHsaJpCTq6Omx6D4Uj+NG2P8JtN9/q3SOb5jMGQBIJfyqNjtZWfMa8mrffwruv/xMfz5yFVEs7or6AcfhIzJPg6AwSzCXxEuPOVCk4C5Am0MqzKoirYngg9qMr2WX53z7yeLPeQIx5JrE4fIkyRONxLF6yBH979VWvmiqZNl+ktbMDPxm7Kw4+fJwteUmnkd+bHNua8HJ1DX8glwBG+s/uvN7AyRsBFY+aHu4BU4UcFpDz5RLIOLv4g2D/zMmTJmO//fdDc3OLBZQI9pKSuFV73XHHHdhowzFFsH/V5I3TNJWU4487AW+/9Taam5uQSiVtKfRwJIKzzv4VDjn44Hy+i6zSF7YpayDJppLoaGrCX8c/ixefeBJo7UBL03KEwp7TySgm+9GEI1Gz9GFWOUVCCITD5oSGQhGE41GUlCZQVVuDaEkcFbW1SFTVmCITj8cQpGTJNVoDXvewCRMm4PDDD8/B0Ycwge33Y9/99sMFF17wRSlcN0vq2tWeNAbwWO6Xy6s/nDETu4/d3Yq2CfaammrEY1F7fcMNN2CTTTYpgv2rBjuBOm/ePIw79DB88vEnaG1tRoaZfUFvdblbb7sdm266aR7sNhV3e1gEk/Igs/7SaSxfuAjPPv447r7zTrS2tZrjWVVVjZjd/BamemPgkCH4+bhD8c3NNjW6FIjSuaMV92o4c2mF1iLaFBrKhh7h9YpDAfz973/HwQcf7OXfZL1gDmnRjjvuiKuuvtocWK/SaM3ThjmzPsLYsWMtxYIDm2WNJSUxLF++HNdcey2+t8UWRbB/1WAnUCZPnowjDz8Sy5c3oaOjzSZtgn3EyJG4884/WQG2KwmuDOzMLfM0aB8oST799FM4+6yz0dWVtFycATl+yxYVO+y4I84571ybOciL6VB6vJzr+njSHB1Toww51Ydc2pQd8M8D+zvvvIP99tvPHEhSE0mc3//+93HzzTeb3GgUaC2Afd7n87DbbmOtFw1nIqZYlJUlrCXHRRddhB122KEI9q8K7IoK0uo++OCDuPzSy83qdnV1eBJd0IfvfPe7uOmmW0wTd6uFun9nLyDh8Wqb4n1ZPPXkUzj77F+ho7PTjDR70dCy09Jdeukl2Ha77Wx0+K020ytiFjXIiRg5haX7NPIFf2Bqw2677WYNjqwLQE7X/9a3voX77rvP/IS1ZdmXLFqCn/50V0uRpg/CVUwqKsqMs//yl7+0QVl0UL8itAvsdBJPPfVUTHh+Atra2o2vh0JcbQI46KCD8Ztzzs0HdP7bV6WebLq9eXNZPDN+PM4++2y0tXfYW7W1dYhGI1i6dBluvvWPRo2kwXsg//e0Vx0uN37yzCZX+WzAosWkZXfBzojvk08+6U01xmTWPI1ZtnQ5xu42Fh999JENOmaKEux0ng899FAceeSRRbB/FViXzk6LyyDJHnvsic8//9xAQ2WBagkpxE033YTtt/em3/8FGDUE8nS7LP7yl7/gzDPORHt7hzmwdXW1iESiWLpsKW659SZstulmxqm/OO7KAOm85yI/NwUsWrQI22yzjTmB2bSXxRgMhjBw4AA899xzps2vSbC7Em5z0wrstddemDFjpilMLHYpLStBZ2cH9thjDzMoRcv+FaD9i6gZMGnSJBxyyCFoa/O68vKGkMawFR4BQ/qxKmB3fwaP//zzz+PUU09DRwdpTNaOQ+mRNObmm2/E5ptvvtrH7X6pCHKCnb0a00lviXdaVTqHL7zwAuIlsTUOdht3Ph/aWlqx//77Y+LESWCagcBOWrjtttviwgsvLIL9K8C6EyIG7rrrLlx77bVYscKTHMXNN9tsM9x77735HPL/Zdnd30EO//LLLxtX7ejosvOpOzA57I033oBvf/vbvQY7E9BIY1hdlUl9EaCixPniiy+iorJ8jTqobmZlV0en0ZV//ON1s+zl5RXmoBLspGx/+MMfimD/KsDu0WpW5mdwxhlnmF5NOsM2EcpNOfbYY3HCCSfkswZXB+w89l//+leceOKJaG1tt2NwvSaqFLTsf/zj9fjOd75jP93NX1/da8FBtffee+Pdd981y64UYg7YFya8YCuJGG1fC5ydkdVjjzkGzz33ggXFShNlqKouNxozYsQIi6IWaczq3uE+2p5AodR45JFH4YMPPkBnp1fCRsAQlFdffbVRBDftdlVPTbC/+uqrOO64442zC+yiMTfccB2++93v9tqy8zccc8wxRplcy06wP/vssxg0ZGCvz7Gqv5mpzmedeSYeeugRK7zmSuHV1RU2W3JWe+yxx4pgX9WL2ZfbKc9jzpyPbepdsGAB2ttb89Idb86f/vQnjBw5ssdgZ8Dn6KOPQWen1xFAS07Ssl9//R+wRS7I0hury0FFLkwqlupKm2NNks7zjR//tPWbX1s6ezqZwiWXXILbbrvDZNSy0jKUlZfYzEJfgrOnGY5ibkxfQvl/HyudZn4LjGpQJaCj5/F1r7nnBhtsYACifNa9NvR/H92jSK+//jqOOOJICyrxIc4usJPGqPJnVY65sm14Hn5PAj7Z2ZUfrATVQw89hG9svPFac1AJ9uuvvx5XX32tNUmiZa+sLLNoNB8vvfSS5ekoqtvT37wm9yvIRDCBnVTl9ttvNxUmk0lZMIQPhtuvvPLK/xpI+m8XnfSCYCdFomUX2Elj6KDKsvdkIK3MEaaGTbC59aZMvtrie1us0aCS66Dy/AxknXvu+WZImIRWXVNp1QO8vi++9BJKEwnv+/TH/neFmuLLZpy8IZTKmCrgtbvI6euZDM4991wccMABqxRM+k8W97XXXsOxxx5nYCcoGD6nL8B+kn/4wzX43ve+16NZozvYp0yZgj333BNUQ/iQmsQYwdbbbLNGLfuXvksqbbGFE044yRx/5sfUGNizNnO+MGECqnMFHL2hbkXLvppXgEDncio77bSzRfi8Tls+47y0jnSmuOJ1Ty0vwf23v/0Nv/jFCXmd3QX7tddeDeavqBZ0Nb9+fnPOIFwTaeedd8aK5U02OFX5xFnr/3baaa2CnX7KoYce5oE9FkdVdYXV6nKAP/XUU17hOquV1oI61JNrWpA0hjfjr3+lDn6yrRznVfSzS5bfigyeeOKJfMuLnlihtQl2Jlox2/DjOR/Z4BQVu/jii7H7nnusNTWGNQEM0O2xx16WKx+NxlBVVW7XlN+R+Uf0hYpg78kw7MU+VC6YY33bbbeZZSc4meVIpYChbWbpqa1ET8H+yiuvmE7f3u7RCyZGMaGMU/pVV/0eP/jBD/rEsvN4TLKaMW26pRKr8xip2H4H7G/n7slvWN3LS87OTmo77rgTurpS9lurqioQDHpgv+eee2y9qiLYV/fK9nL7ro4unHzyKRbl1MrU/qBXFkf5jLRgXQA7BylnJqY7vPPW2wZ2dek67bTTcOi4cWuNxhDszNXZdtvt0dbWYXlAVGPC4aDRGBoX+ileHeqaT0zrCUQKksYsXbzUNHAGk9Q81B/0WwPTW2+9FRtttFGfgJ2cnUElWtY1YdkJdjrXnEEmPP9C3rLTF2D09qhjjl5rNCabztiCwj/84VZoalqBcCiCispSRCJhe/+yyy7D9ttv36/XVioYsEsm44j/9OPPMG7cOHz66af5Zv5M6d1wzIZGbRja783UTwsrNYZpw5wlBHZaOdGY3ursPA8HK1OJH3/0sS9Z9qOPPhonnHSiGbjepCSsqoWkZed32WqrbbB48VKbYSoqSi2tmXIrYwE//elPi0GlVb2gvd1OOexvvfG2hdkZ4OF71qQoFMCuu+2K3/72t70O9qwM7AxQkccK7D/60Y96rPboOvC7E2B0Ru+9+578wCVvP+igg3Dm2WetNbDTQaWjv912O+Czz+baNS0vL0U87smtZ511lqUA28Ar6uy9hfJ/319NhgiQe+++D5dffrk5p3m5LujH7353Of7v//4v3waup9+I58inC7R32jkqKisQi8awvGk5rrzq91/Ku+npefib+Ec+fM1VV+c7DRPsBNYFF1641jg7wc7HrruOxeTJU6xvO7MeWSjO63zCCSfi4IMP8mZMr6qw3z0KisaIyvzyxJMt35vOKakErVBpeam10uAaqL2d9pUucOQRR6Kzw4ugyrJzSr/iyt9hO5bl9VIpse5j6TTuv/9+nH/ueV8CO53sK35/xRqNoLpoFdgPOugQS/NlJ7KSRByJRInNPkcccYR1QrBikiLY1/xAJzCoXuy5+15WPsaboIKHzb+zOW6//bYvdfHq6TciCN9++22MG3cYOnPSI9tVM6pIqfCy311qYF/dopDu34eDir+JWY+/OO74PNipKm211Va4/oYb1loiGMHOYqrjj/sFnn/+Bct8JNBLS1mt1GmK0XHHHeu17WORbT98FIxlV0daFjrsvtseBnqCXUvDHPeL43DUUUf2CcclCLlg8MEHH/IfwU5loi8sO4/xr3/9CwcfeFCu6ZK34gezKm+97ba1BnaqMRx45513Ae6//wGrPE+UEuws4OjCvvvtixN+cYL10elHrR6/NOQKBuxyTmkFT/nlqfnlX0hh2I7uD9ddi+9u4eWY9wWN4YIG++yzL6jp8+Fa9ksuYIq3QwAADwhJREFUuzjfWqI3qg9/EwcxVwsZu+tu+QXGCHY2Jbr73nt6PXusqgE2y57N4qqrrsENN9xoBRyJRDwPdvoQJ598sgkBRbCv6lXt4Xbit1dddRXuuuNudHR4xRqkMQ0NDfjTPXd5/QktDbV3pJI3fdasWdYhS5x9TYCdl4J9bxjM2XGHHxtF4m/ibPX1r38dDzz4gOnavRlQq3q5WajOaiXms1/xu99bAhhbh5SWlVp3Y7b8OOPMMy19oAj2Vb2qPdyOYCd1YeT0tVf+gXYDO1e8CGGzzTbFLbfeYk2Lepucxa9HsFPD32WXn6Kjzesu4Ors5OyiMb0dWKQOVDu22WprC8vzXMyuHDNmDB546EEbvGsD7FzFhI8HH3gYF557gQE8VhJForTU6M0uu+xi8QA/m6UWpcceongVdyMI2JrtqKOOwgfvTUEqzfxvLrgcwrHHHoNjjj0mH8buLQB5LrbU23mnndHW2m4AZLcCFkIzmnj5FZdZxX1fOKhyUn+y085GZ3hM0hhmbT70yMP5hLZVvEw93oz1AHw8+8xzOP2U040mRmJhlJaV2e/faaed8Jvf/MabaYpg7/F1XqUdaV3YG+bAAw/C3M8W2DTLJCWm9d5zz934xjc3zlvA3lpCziJsb7HD9jvkwc7KHfoGBPtV11yJH/7wh33iDGsm+dn+B1jBCB8E+9ChQ/Ho449ZIKu3g3dVLnA2tzbqKy//Dccfc3we7LTsfHAmO++883K9bIpqzKpc0x5vQ7C/+eabVj3U2swiaOZ++62hEPsysrW0Hn0Bdurp22+3PVqavcamLtiv+cPV2HLLLXtt2fV9aTlPO+VUPP7440YZSF2YqvzIY4/aedcm2N9+8x0cMe4Io1bhaMhoDL8fpdYLLrigCPYeI3g1dqQjxz4wl112OTraPH2dNGb33cfioot+m1tWpW8sDm8uLfh2222PpmVN/wb2a6+7xoo3ektjXLDfcN31VkrIgUWFafDgwXjo4YdRWVW5VsE+bcp0HHLQz7F82TKEoiEbbLweW2+9NS66+GIvFaNIY1YDuauxqS3olVtm/KSTTrIqdzeYxNz1n/zkJz2uN13ZV9H6qD/e4cdYMH+h3WzedHJ2KiZ/vOkG6xvTF86waMxjjzyKU045Jd8OhGD/84MP5DuarcYl6/Gm/J2MY+y7775YwiV4AiHzVfg+8/cvv/yyXGfhHp9ije64zuvsAjunVSoCbAaqqZ4t6VirSWdORQ99cTV5TqoRP9n5J/jk40/zYCd/piJ00y03WpesvgT7G6//y+pm+dv4W9hmmw6qMjh7S81W5boQ1Cx33H333a09SSgYRnlZuf1+5rL//vdXFMG+Kheyp9soAYxLtLN8jSqBlkJnmdidd95psmBfAU+WlrRpt113w8wPZ+XBTkmQ57/ltpvBttJ9SWPmzJptiodmLcYMSGMaGhvWivSo382Zi9VetPB+X8DAzgfb/V111ZW2ykg/rd1Y9xcQU5rA+PHjcfrppxvQJc8xv5p51u76oz0dVO5+kgP33nsfTP5gsoGdFIZgJxhvv/M2fPOb3+wzEPL4Cyh17vwTk1f5exgo+/MDD2DAwAFrhbPz9/NaM7mOMwy7NvjhNYglT2dE95prrkYoHC4mgvUFyP4Tf+b7TOmlg8q21LTiKsEjtZFT11ffgcejZT/wZwfivXfft+NTdhTY77r7Totw8tEX9IJgJ0fefexYs6gEOy07wT54yOC1CnbSKGY3MsXZl/VbmgTFANafXnfdH4pg7yuQ/dtxuKAvrU1nJ3550knW3qIrmbQVKWhp2ZKanbr46Et5Tnk4hxx8CP71+hv/Bva77/0T/t//+399CvblS5fhZz/7mVX4y7IzN2b48OF9+tv+073Sb+bzmWee6fV2hN9oDMHO33vDDdcjHKFl7xvVq69xs247qFlvamWlzLhDDzUg0JJyRRdmBbIET6VxfWFhdfF14w8//Ai89rfX8tKj1jm99/57wNUx+tKytza3WN9KxhL4m+h8333P3Rg5atRaAbtojGZRXltadqpQnNFGjx6Nm266EZFopJgb09ejVMdjNh4bCZFHUomxErxwyIqUOd32tg50Zd9bYD/2mOPw0osvGdjJXQX2Pz94vzVN7UuwczGAX/ziF9aXXWD/0913Y/QGo9ca2PW72X/y0ksvtc7Cklw5w9xyy81FsK8poPO4LARm/3ICm0oBwc61RrkAQV+0oPtPYOf7J//yZDz7l+fMKeZNp/RIB+6Rxx7GsGHD+oSvy6KysSmt6RVXXGFgJ2248eab+qTyanXuDwc2q8BoTFLJtNEYSqEc3OzcEItHi5Z9dS7oKm+bBdIpr+Emg0cEHS98XUO9Ne2xdmy9TOf9b2DnmkpPPvGUnZcOKiuVKD0+9sSjGDRoUK+lR1pSPVTdz36L1Lp3GzvWFiNQC7++pGn/7frzO7FwhYElpsvwd3OQM32BzVajsWhRjVllAK/GhjatpjM2vdPa8DUt+6abb4ZbbrnFgM/Xff3QdM6uXA8/+DCSyTQSJQnE4jEkkx147InHbaD1hc7Oc/E4XAyAyW3mk2TpcOcWJ3OXae/rH7qS49Gye+nNu6CjrTO/sjcH95133WkF2MV89j68EXmLxyZCHZ348Y9/bCm34si/POVkKwBWi+c+PLUdijecj4svvgj333s/ujoziMXiKElEkUy144knnzYdvC8DWTovf3tPVgvpq2vA81MQYApz07IVebAPGDDAFnjgomZFNaavrnaueEKHmz1zllkZ6t4EAa35Pffdazp3X5TgrexrK5B1xRW/w1133IVkEohGWMgQQyrdkQd7X1j2PrxsfXIogp2BM4J9wbyFRmEo87Jrw3333YtYSdxbkKAfPtZZ6VHW9ZGHHrbUUks5DYeNO47/yzPGZdcEX9c95PkZHr/15luRSgHxWAniJRGkM5148qnxdvM10/TD+96jr6QZlc9Mrpv14SyEwxHj7YxnPPjQgyZDWhPZfvhYp8FOwF12yaXmjNKyE+As/D3/wgv6nEK4907pAjfe+Edcf931SHUB8XiJ0ZhMNoknnnzKIpyFDPYDDzwQb/7rLZNbCXb2pyfYS0riRRrT1wNdfRBZ1MCV49T564rf/x47/2Tnvj7dl46n4u477rjdOnV1dXHZlZjRGPhSePyJpyzoU4hg50Dn72cngb+MfzYPdsYZuM5TWXlpEex9iT5Np7zof/zjH21hK1p2KgJcQ6kvNe6VfW+en+e75+678bvLf4eurqytRCGwP/X0M2bpCg3s/D0CO3tmsv+kWpWwI9qjjz6KkkSiCPa+BLsuOi88gzhcSYN9XBhOp+S3pivuBfaHHnwAF/32ohzYPc4eDME4O9OKJRv29W//Ko/H38S4AvtPsnpKYGdC2MMPP4yycm/V7f74WGc5uy4ms/Bcp3FNO6audXvs0Udw3nnno7MjbQ5qLB5GOOzHU+OfWWu1oWsbVPJXuKL15ZdeZr4ROTv/Hn7kEet5af0e+2FS+zoP9rV9s3m+fA7900/j17/+NdrbkiiJM6gURiQaxNPjnzH9uVClRxqYJ598Er8662z7jZQemS7BdZWqa6rXWrPV1b33RbCv7hXL8Vbe8Beefx6nn3Y6OjrS5qCSxpSVx43GqAywP1q4HvzkL82etO5c5PekE040qibLzrQNBtOYddoff3cR7D2483KQJ0x4Aaefejqam9vzlr28ogR0UOk3FKKDqpmNxRvHHn2c8Xfyderrf/7z/V6ZYJGz9wBV/XQXBbRee+1VnHTCSWhp9hbUos5eW1uJRx9/Ip+T0x8tXG8uq9SYiRMnYtzPDzOBgJSNf+wjP3DQwGIiWG8ucH/cl9Ljm2++geOPPR4tLZ2IhCOIxkIYMnQgHnjwoa80f2VNXy8CfsaMGdh3n/3Q1dllVp1gZ3Bv2PChxUSwNX0D1ubx5aC+9+471oFsRVO7cXaCffiIwfjzAw/lv04hWnaCnYUyXPSBNQQEOgFPsA8fMRzwedmZ/e1R5Ow9uCOayidPmoRxh45D0/JWW/GZNGbkqKG45977CxrsHOyLFy82sLOdNtUYpg0w63HU6JFF6bEHmOrXu/CGT582FQcfdAiWLWuxCCqlx699fUPcetsdeee0P1q43l5YDnb2utxzj73w6aefGNipPrFcb4MNN+i3kmvRsvfwzhPss2bNtOVflixeYfns1Ng32/ybuN5WpvCm8UIEO2VXtizZe++9bVEGgp3BJQaauKByf40vFMHeC7B//NFH+NkBP8OiRcvzlv173/82rrzqmoIEuS6V2v+dccYZtrgZZVZmebL7GtvyFcHeQ1D11914w+fPn4d9994HCxYsMwc1HAlgx//bHhf+9qKCBzt//zvvvGMlkQQ7uxaff/75a21xhJ7gomjZe3LVcikDixYtxD577YN58xYb2CPREHbdbSf86tfnFDTYdckYUGKHMj7TsqsVXn+lbkWw9wLsS5cuwd577o3PP19gYI/FI9hzr91w6mlnFDTY3RRrN7NT9KUI9h6Cqj/uppvNBb322Wcfs26MoHL1OFbwcGrvrze8P17PtfWdipa9B1daYGdAhYrEnDlzTGdm8fFhhx2GI488sgj2HlzXNb1LEew9vMJ00NgQac8998TMmTNNZybYjz76aIwbN64I9h5e1zW5WxHsPby6kt/2228/61XOih2GzNkW7pBDDimCvYfXdU3uVgR7D6+uiq73339/vP3225bTTcCfeOKJRbD38Jqu6d2KYO/hFVYyGHuVP/3009bGg4A/55xzsOOOO9rrQqxB7eHl6he7FcHew9sgsHPV6YMOOsi6ZKmTLYsZimDv4YVdg7sVwd7Di0uwU14kyJkfwsQorsrHguO1UfTdw6+9Xu9WBHsvb7/bEo6H6q95Ib38mQWxexHsfXAb812Fc8cqBpT64KKugUMUwd7HF7XolPbxBe3DwxXB3ocXs3io/n0FimDv3/en+O368AoUwd6HF7N4qP59BXoNdjln67tT5jqphXgtCuE+rzbYuztghX6Tu9uqlTmg64Mas7LfqGuxrgyE1QK7WkgwaMKgCots1R1LP7yQdWZ1sO2+gJeuQX8vXugNydC91zHcgnJ1Ul4TCyz35jt33/f/A3lb7IWxiW9BAAAAAElFTkSuQmCC"/>
+        <xdr:cNvPr id="1034" name="AutoShape 10" descr="data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAALsAAAC7CAYAAAA9kO9qAAAgAElEQVR4Xu19B5icVfn9mV52tvf0CuGvohQVRaXLD0QIvUiR0IuAdFCpUkWagPQiTXoNUgKIoCKdkE4KNb1ttu+0/3Peb85wWaMmu5uwmczwLJOZ+crM95373vOet1xfNpvNovgoXoH14Ar4imBfD+5y8SfaFSiCvQiE9eYKFMG+3tzq4g8tgr2IgfXmChTBvhL3fOUeexb8798fvn9769/fWTmess6GfuRe8BSreoD1BqZ980OLYF/JdVyZPrUyoBsmV4r/VRW4fN7+PsDnKyK8byD9n4+y3oN9pbDMrJoFN6z7u22bBfzI/NsVX/kRCXC/t23RsK9prK+faszKQgvue1lfhqbWu/hm5r1/Z7M+xwJn7V2fmWYPynYM+6f3CV/wLbPavi+Ok7HtsvD5SV68IwT8ftuf//YXrfwaAX5BWvYvAXclnISf+/2eRTUMAkin0w6dSHvARdYDKgFLIGYyBtD8ILBNMjkc+5BKpezPn8ki2dWFVDqDTCaDdDqFjM0WHsjDkShC4RDiJaVAIESkAwEfUW6DpEho1gjWC8GyE0BfwCPryyJFcBI2BCcB66HTwJruSqKjvQOdbe3oam9HqrMDXZ0EZsre7+rsRLqtFV0dHUgmk/aXSiaR7uhAW2urgbmjo8MGR4Z/qTQymTSSXQR60kAdCvgRCAQQCgZtcHiDIGnvhSMRBINB+H1+hEsSGDBsFAaOHI7hG22ESGUZMgE/gj4SoaxHcLI+ZPx5srNmULCeHHWdt+zZLPmxL0cXgAzS6MxkEMoCgXQaqdYWfDxrFqZ+8AE+njUbyxYsRLoziRD8KI3FEA4EDIzhcMiOEw4H4c+mzb6GQiH4CVy/H5lkysAdDHE7byag1dcfvwBtNwdCMBBAR2enDTJuzwHEcyRTKRsA3C4SiSAQCiHrCyAUi2POwkXY7ecHY/Sm30IoEkVnNo2IPwhf1odUzvAXLX7vRmUBgD2LDJkGHUNfFtl0Epm2Vnwy/UO8+9o/MH/OR/ClkiiPxRGPxswSk5KQN7e3tiGbSiMSDtv+gYAfWZ8PndkuA7HoDq07wc7XpCUG/hw9IogD/oBRfH5GIHNQfEGlfEaZkqkkurq67H1Z9nQmZRY+GosjUVOD5ekubPitTfD9n/4UkfIyA3og6zfLbrS/d/d6vd97nQa7AJXOAS2QzSDZtBxP33kHJr/1DjYaOgLo7ERXW6tRlNaONgSCQaMS6WwGTcuaEAgEUZIo8ZiyD0il0mbN/YGAWW/j6YbkLMLhMDo7Ow2wpCR8EMh8TUtNq85tu1t9fs4BYw5obpBwf3J5EhYOkkgsjpqBjUhU1yI6dDi23nUXIBTxqIyBPecrrPeQ7fkFWLfBTqePAKVlTyWB5hb8+fo/4pP338eQxgFoWbYMHW1tyKSzCISC6EqnEAoFzSoT0AQucUwQ01oT4LTUBL5pKTlQE4yZdMYALuCS4hDYZulzwDcnV85u7p5wGx7fBk42a8enZbdZIpuB3+9D1o7tRygSxpDhI7CkM4Oxxx+Nktp6ex9+Osre4Co+en4FCgLstOzoSmLyy6/gvquuwYiGRqRTKbS3t8MX9MMXCBhV6ero8pzKdMZUlDD5dKoNUdKbdMo4OwdDV9pTa2ipjbf7vYFBUPPfoji87KQmBDMBzPOZT5mjO9xW+3MfHkOzAUGfphMaCCFLXyDoNz5fmkhgwKARWBAK4JBTfolsMAD4M/D7gj2/y8U97Qqs02A3K5qTtn0tzbjq1FPR/NmnqC6vRDqdMepAxzMcoeUOoKOj05QTD4xZxOMxj2dnskhn6JSStwft39xGdIRA9iTEtAGez/wjkAVegl5W3maCHP3RADHeTlWHgy3jBZ14Dp/fm0c0MEpKStDY2IhW+LHVgQegdswGCNAf8QeKpL2Xg7YgwM5rsGTmLPzmsHEYWFaCWCSe58a0ugSl6IfASiubSCTyTmhbW5tZbH4uoAqUBDs/M4pD6sKBkEohGo3aey4n57m0nzsTcD+Bnd+X/3bPxX9zm0SiBJWVFRg4egwCgwbg+7vugmzWjwAtfPHRqyuwzoOdwKOhfOPp8bjzkkswvL4awSDVFc+JJCBlgfO8OU1dvMveF/jNwueCTeLUsu78TO/lAe9szzvA9/nQ8bi9rLcCWJoR+JozgXwAzQjcJxqNIJGIY8DI0WgJBTH2sMORjcXykmev7vZ6vvM6D3YDZDKNx/54E16+9140VJbCFwiZJaRVp/WWZea9JrAU6STYTFbMOZmuyqJtCVDubxw7R1+4n94ThxdN4WecNfiaf6I+whlfC+zuIBGNiUbCRq8qGhuRDkXwg7Fj0fC1jRAMR4rSYy8H67oP9kzWtPN7Lvs9Xn/0UQyoq0SA6gcDS6GQgT0Wi9m/XZ2btMU4PwNPjlU2Hp3LTREdcT8X1ZESo+vP1zy+9pUyI04vYLvyI7eR46sBFPD5EI9HUV5fi4aBQ7GgM4n9TjsZwUgR7L3EegE4qGnmpqRx12WX4x+PPYHGilL4/F6UkiCnw8c/WmKF/wl8KieiLrL0fF90xbXsAjZnCllrUR6+dqmN65jq+AK4tHYdQ36AAk1yiCPxGMrLy/H1r2+M92bNwc/OPgNVAwYUHdReon2dt+xUXZDpwv1XX4sJ996PobU1CIUillRF8MbjcfuzqGVOQiS4ZOXlYMrycoCIqwvwepbVFnXha/5bSo2suWYHPUuBEegViNJ+7vH5WTQeN+4+ZsMxSEXjGPr9LfC173/fYgJfShVmukIvAbA+7b7Og50SYjbdiSduudV4++DqakSjcfhyyVhlZWXmpMphFLhlRQl60RSBTo6jOLyinnptmY05i07A0uJb2oAjS7qcXVKkVBi+1oChtRedkiMdDsdQVlWKIQMGombwULSVJbD9fvtbUhlz3pT3puDX+gTY3vzWdRLsAp+ndvB/SfzlzrvwwLXXYUB5OeIlCUsmkRpDy06LLUeVPFmOqaiFLqLoiSy9rLcGgktB3Agrz6WBJFojNUbHJMg5uPhQWoHOr1mDAzMeS6CkogTVFeUYOnI0Pmlpxp4nnIQ0Z5JgwAM7/11MB14t7BcM2F958CHccenlqEskUFlZbekAfBDoBBBzV1z5UGB3KYsrDSpKqmioVBk3cCSu7c4Iokd6z5U9ua+iqMqW5Hv8LnodCoQQCUcRLY+ivroaAwcPwbS5n+OQcy9AIB63IBTTzZiwRrAXM2ZWHe/rONi9aiBkkvjXM8/gpnMuQH1pAiWlZXYFCHA6p6QZfHZphHi0q5oIiArwCLAEo3i2S2n4HgeQBok7O4jqyLprRugufYrC5KkNfIhEoigtT6CivAwDBwzE/OXLscUBP8PwjTf20h+ZT+Njnr4H+OJj1a7AOgn2L/00SxdI4p0JL+KaU84wsMcTpQZw/RH0VDcITMmDBFdLS8uXMhgVdJIWTmAzP0aRTgFefF3URZ9rFugeoJJ/oAEmC69B5Tqw/IwDk5Ip/+rq6izvvbW6Cnsdc7RVNtn38LEwpcjaVw3m3lYFAfYMkpj55pv43XEnoSIcQqKs3JQYgltae2lpqb1Wiq50cQWARGdcTi2rK4dVVlp820CXy1+XE+o6n9xe0VPJjJo9ug8MNy2Yg5Q+BsFeVVWFxoED8eqMGTjzmqsQiJXktHzGA+wWrs79Xq+3XafBblIeA0NI4fMpk3D50ScglkqZZSdXJ0hp1flvAsd1DAk+Wm2CTxq8JEkhQjxaOjupiXJf5HTKqruzggaJnE4dh/vwfC5Pl4Kjc/I4/M784wCtrKzEiJGj8Pwb/8Lxl1yMqsGDActtL4J9dUduQYA95Uth6UezccEhR8Df2oqysgpzSmkhCXTSAsmP3Z1UWXYCmVad/FyJYwKt1BXu684O0tFdwPIY3N/NbpTM6PoJPGb3hDH5Bu4gJdiHDRuOqR99jK0OPgCjN/82fKyMkuJe7ESwypgvCLAnfSm0zZ+HC35+BLLLm8zBI9BNxovH83xdeeeysLxKoi0EIlMICELuJ2dWOS9SYaSfS5vX+6JFPIcVabPmNJk0Cy3aI2dYUVZRH5fLK/hFGsM/xgkGDhyIQCSG6AYjseVuuyJrtam5tIYii1k/wC4OnUIGnUuX4lc/PxTpuQssTZYBGAKNwKWTR9BLfpQVl4oiYAqkbm6MJEhRIDfEr/fcIJS4tzR3RVgFeAFcn7vAdzk+Qc/vTCpTXV2N4SNGYH4gg52POAIZOqk+f1FnX2WYF4iDSiudQhaZ5ib8etzhaJ39McpKE1ZiR4CRwtTX1xtoFFgiqLuSSXQ67TKUb+5GO90opwJIypQUR+f7Lm1x+bmSzJT56EqUipxqEOi4yoHnMcXda2pqsNFGG2HykoU4+OyzkA6GjLeTzBQN+6ojfp2mMZ5lp4Oagb+jHb899jgs/GAK4rEYIlHPqtM6kvfSQeW/3WILOqiSF2VhbfDkCjJk1QVSOadyWBUMcqVJl7+7aQW6JYqYKmWY77sDTLOKl9vuff+KigpsOHoDvP/5pzjivHOA0jIvhbgI9VVHeiFIj54ak0WwqwNXnnI6Zv39n1bHGYl5UVMChryXVIB8WlSBQGfmIzm75EDXISVo9dp1HEVdJFWKh8uiS2p0+bnybzQodFzNDhoAbsEHB5aCYVWVVRg6eDCmz5+Pnx5zJBo2HGNdxALFjgPrH9ite1ZnO26/8CK8++wLSJCfx6IGdP5JwlNlkhxUlckR9AoUib+LTgiQckTFyQVYXW0pK92vvhQbpSco4OQGktz8HA0anp/fl9+/orwco4YNx9JUGrUbfwNb7TGWJVHG24vGfdXxvs7TmHzP53QK91x5Jf5234OoLI0jGouazk76QsueSJTltXepMMpvF01R0bQA7QK4e82owC7a0j2dQBSGx+QM46YBd58V3HwaObsEvWvdR48ajnhZJWY1Lcfh5/wGqVCu/UdRelxltBcM2LPpFJ6+7XY8c8vtqEzErCxPnJeALylJoLS0LF9JpIINUhjxZ/6bwCNwBTqlDsjCuzRGfJvPoj0EqQpDZKVdXt7dssuJdbMpdQ6BvbSU7TUaMWDgEPxz6nSccPklCJZVIsDOBEUPdf0DO9JpTLj/fjx05bWoLi9BMOQ5ePyjIlNZWYWysvJcew0v/7y1tdXALwvPZwLezY2Rk+o1VPKKNbrnysipzEuhTr2qm92oJDIOKDfopHwdV6vnv8nhLZJaVoqa2mqMGD4Kr0+eioPOOB1Vw0fAHyyqMauM9EJwUEVj2BHsrWefw63nXICKRNTUGAWWaNkrKioN7AoKEdjqxitVxg3ni6YIyPm+MGyrkatdVdG1BoSsu2iSAk/63NXW3VwaV8ZUGgL34fFUNF47oBZDG4diflMLNh27K0ZuvpmlMRct+6rDvXBoTCqJaX//B6477SwkokHES+JmiQX4+vpGkyCVaUiwkW64kVOXS0uCFAXhdpIaxc/F12XpZY35rBlCt8JNFdB5LLcn1wdSg0sFJgI9ZyYO1vLaCgyorEdpbSNio0Zi0x1/DB8te5HGrDLaCwDsuR7/mSTmvPserv7laQimk0ZdCEK2pWCXr8GDB4PBGVdVobXmH9ME+Mft3Q4Eoi5SUrrTFUVH3SipuL72cdUc3hXlxLhZj64aI/VGEiZpDINhpRWlGDxgEBoGDUNrLI6tDzwACAeseMP9Xqt859fDDdd9sOcqkDPpJBZ8+CGuPPlUJJc3WRRVDh6tI1vKybITkASdyvNo4WWJ5UC6z24KgFuU4SoxArwwpAgpn/ONTHNVSd2VGQ0McX7lx2hgEuzl5aWorq/FkKEjsSyVxa4nnYRMyAdGA4pgX7WRWzhgz6Sw7LNPccWJJ2PFp5+hpsYLIhE4tPK1tbX2J8ohmiKtnc6qW4zt8ms3CKRIq8DN7dSlV2kBoidSdvS+jqmorbaT9Olq+Do+32MEtay8DFXVlRg6ZAQ+a1qBA848A/7yUm+FkSKXWSW0FwbYrX16Gs3z5uIPZ5yNBdNnoCrHzwl26uwNDQ0GGqkp7I3OXuySHemkSo6UoyqlRiAVzVG6gNtjRrTEtfCy7m6GpIo7rMNwrpe7m/0o4OozHoNVVpXVVaiqqkRjfT3mLW/Grscfh5pRI3K57UXArwra132w59aqyyCD9oXzceM552P6P99AbXVVvlpJYGckVX3VZeElAxJ8bpRT1rY75SBwVXcqXi2gC6ByYJUy4JYCKlClc2mwidtL0ZETy5vI711SWo6KigQaa2qRDIZQs/HXsdVee3rpvjlJdFVu+Pq8TUGBPbliOW78zXmY9PLf0FBXm29cSq7O8jb+idrImiqoRLC7ll3qiWiO+LkALMqhomtXydEAEQd3I7Iu2N0Bxfd5fll2pS/wfcvYLImjNFGC2ooq1A8diokL5uKEiy+CLxy1dtZFKvO/h/E6D3Z1yMpkUki1teLmCy7CxOeeR601S/qiWknJYHT2+L4AqeokJYQJdASitHVeRpdDi4PLGsuhdOVJApcDRM6wLLnL5zUj6DhSgjRjyBn2eslEUFZegZqKagwbPRp/mzIRx/72HJTVN8LvD3vL0NhialzDtbhwwcqgXzBg52JcmY423HbhJZg04UVUlntF1ypeZtYjHVWCXj0bu6cMUH4kAEU73EalruXVQJH1lb6+Mi3epUGaTdzqJ3dwuSkJSiPQTFRaEkMsUYqaymoMGjoUHy1djG0O3BejNtkU8DG/3QdfEez/1byv+2BnYMYHWy3Dn+rCPb+/Gu8+NR7xaNT0aSWDkcLQQRVvl8Iix1SpAnwt+kEgurKgLK9oifLbXe2+e6qBG0zSOTWgNBDcHHelF2hW4cAwyx4NI5ooRUVpOQYNHIxAWSlKNxyOH+76UyAYRZaVS9Zeg9a9aNkL07LnwJ7KpBHKpvDQdTfiHw88hDDXJ8q1z5BFp/RI/i5+S7BJa6dV5zqltuhvroe6opvi2aI8ojFu3osGiCKffBbP5/4aKHqPg0pWXb1ppPoozViOJwNLiVgUoUQJSksSGFQ3AHWDBmNOVwsOPe1UZEMRZEiZ4C1yDFPfi4/uV6BwLHs2jWA2jWfuvBt/veteZFJJoywqb6N8N2DAALPuUlMkDYqvU2t3ebpoibR1qS2uI6mIp6Kj4tnaVtRE8qPL2fWeLLsrVfKcKubgACmJRQzsJfEEGipqMXDwYLz56RycdMlFCFVUAgGump2B18mmCPaCtOwsyWPun1EJXwavPPIEnrvuZiQ72lFdU41QKIBQOIDyiioMHDTIrL0bEBJVURak0nMJMDcLkhdPujrf7y5BSlnhduLmuuDddXRtq+Poc5e/K2FNFMmaJpUmrHNCVUWlDdyPP5+PLfbbE1/bfhsEbM1uLkhWXEbyP81p67xlp77OlaBtTVFfBu88/zIev+IatK5osoW4CPZ4SRS1dQ2oq6+3Ag5lIYqmELi06GyHp9wVBZR44UgzlG8u6VFgl9UXjxdHl9bOz11ZUhZfpXpyRHUcRV1Fg3gezU58tjyZ0lKLBocCEXweyOCoC89DOFxi7TWygSxYnVp8/PsVKBywG+gzmPHPN3D3+Rejefky1NbVIBQMIBaLgFmPTAQjf3cLp13OTlC7zqK4ujsAxL0FdtEYV0kRPZGVd7V53QJZdYG9e5UU3ydX5/ta8U/KEp/ZHmTIwCF4dcokHH/5pageOAhZP5DxZREs0piVjvV1HuxZk9volnHF6BTmfjAFN591DlYsX4qq8grEouybSLA32J/aaYh3C+x8rSZJUktENxTllGPrvpZD6jqosu4aLHotvi66ooCVq/poH9EmzRikVaRR/P6cNWjdNxg5EnObVmDLfffB13/0AyvCTmezCBZXwy5csBuN8XGJyCSWzvwIN571ayyaPw/VlZWIs6VGJISamjrrH6MW1rLEqlJS5qOriLgUozuvliOqgFN3sMviS8t3HVcda2UziavFu3RLkVothkbr3lBfh5oBg5Cpq8Wuh42DLxwywBdpzMpJ3Dpt2W3RDa5dyhbt1qI/jZb5C3HdyWdg/qcfo7a8DFHmg8fjqK6usWQwyZHdwS4Lr8ajsrauVXZpjZZu756XIn7Obd2QvwYRPxe9kTMsvV3PmnUkU4q/K0imnpOVtVXYcNQYfLhwAY6+5EIESsutY3sgtxBDkbd/+QoUDth9GSCbRsfSZbjpzHMwc/IHqCktsXySULQE7L3S2NhgVT9KyeWlEHfms2ntyWR+9WnXKruWXOV8Ar+yIOWUysobDeKKxLml4bW9QK0kNPc8blGHmyfD912wcyCUV5VjxJDhmLt0Gb67zx7Y/Mc72kqB/lz1UjFfpkDBnvVnwQKOdHMrbvv1+Zj45r9QznwSdhYorbAksNraGkuXVZdegkGOIQFHq97c3JzPIhQI3WxIpf9yPzc3nsdyS/64naw59+f2GgSiJyoYccGuNGJuq6CVZgPl2vCZA6skGsXwoUNRWl+Pz7o6cfR558AfL7G2eO7+RQvvXYGCsux+ZJBubcO9F16G1195CWXRiOXIROMJ6whGuY6BJqocchZlybVIAcEubVtlewSWrLmoiUtLXCdVs4XAJulSdEiJYfIHXCdY9EURXMmWGiSqT1XXgYjfj/KKCozZeGPMWbwEY489CvUbboCA30sXUEJZEewFCvZseyeevOp6vPSXpxEL+FBXW4tIrATl5RUYMKAxv7x7d7CrwwCjqBwAStbi+1qsgO+LGmh7l8oo4inQCqySLkVRXEvu+g76vHs2pMAqsHPAWHezbBbRkhiGjxqFmtoBKB09ElvutRuCUW/9qCLYC4zG2AoUtq6SlxeS7UrhhZtuxwuPP4pQNo26ulqUJMrygRjSGAFBNEY5L6IbruYtgLu5LYq2ynqbJbZ2dL48dZE1doNKkhwJViWcaWbRTKHtXeBL2VHk15bPCYbsN7NlSF1tPUYOH4VPOlpw1Hm/QaSyxsuC9HutT+kSF5sQrOM0xh232Yy37Eo2lcbLf7oXEx58COm2ZtQ21iJRUoaqigrUN3gOqpvAJc1cagxByD85ne4AkGUluDVAxNX5XUQ/FCUVb3eDSuLrArkiqYrmSlcX2AVwqTtKQjM6lM0gFo2iKlGGoaNHosWXxpgtvovt9zsQ6VDIIB6gLOuH14VgPecz6zRn/3ew+5BNpfDPBx/Fs/ffj0xbMyrrqpCIJyxbsLauzhxVF+yiEZIB1VZD6QICqlKBVcMqFYdgVX92KSYujXE5uaiRrL7WdHI1fJ5XtEcA1+cagJI7swEfYuEI4qEIGhobMWzDUZizeDEOv+B8xOprCXUEGVYt9j9d9x3U/wT2tx5/Cs/eex+SLU2oqKlELBpHOfNJ6uos65HSo+iCG+AhMAl6Al5gF/AkE2qgSEnhPuoMxu9D4Avs2pfbKKNRygqPI7BL7ZETK+uu2cKdNTQATOb0AaFAEOxRRml11OhR8MXjGLP9dvjWjtvCF4ogqPU51nezvq6rMf8J7O888TT+cu99aFu2GBW1jKLGUVleiZraGstnZzGELLrALuWFIKaTKhohNYXPcixd8EmCdPVxcXlt7waaZOkJdjdVQXxeer4c6O7HVYCJ25OT008gK2eC28DGAdjoa1/HvNY2HHLO2QhXV3vL0dCpKSaHrdvS438E+5PjMeGBB7Fi0XzUNNYgHIwiUVJiEVTSGEqP3cEubi7nUzTFVVBkeXlelezRwrqLGbhKjhvUkW8gyVHOMd938+r1b5er63dyWznXbiSWKQLBSNj8kg2GjUQy7cPArb6HXQ89BP5QKF/Qsb4b94Lh7OLB2XQak5+dgBfuvx+LP/sENQ21iMVKEAwEMGjQoDzY3WimrCoBTArjluoJ7KIaeu2CXQEjN69FYNSgEvcX6AVyNy1Big/fIx3Sa5fri8bo99pnVtztRyJRioH1DRiz0dcwefHnGHfWGWgYORr+YAQ+y5lhnSrnAa+UcX1bpqYgwT5twst48c8P4LOZM9A4qAGxklLEIt6qeaQxWhyAgHHpg3rH0FK77fBkyV3e3d3xlDzYPYVA2+lzBa9k4Xls5dm4A6o7fdGM0Z3m6Ddwe9Kz6qoqjBwxArHqarTFQhjHzmHsSx8MWQ4Ra5hsxY718FGQYJ/1ymv4++NPYPbkSYiXxVFZVWNLtTCKqu4CblKXpERxaDmq4s3ctrskSdDRMZVVdxUe8WoB2lVbNLh0TjmqsvhugyWpL25wqnt01eX23JfdiwcNGISRI0dg7rLlGLnlFthl3CEIlLBVng9BNlTy+c3Cr29aZEGC/ZN/voF/PvEUpr37NkLxMGrr6pGIl9jiueobI8VDgNRiYsoxF2eXouJmKArgbi8ZN49F6QPdI6h6raCVCkWk2ZvT6fNKDBVkktLTfcBosLqONN8LR8KoLC/DwPoBGDx8BKYtmIe9jz4a39xmG6/vQMjrILa+RZpsZs2KXBbAtGZWLp3G5/96C28/+xwmv/Um/GE/6hsHoCzhLZ6rFF8pKuLM6gzGY6jyXykBLhip1IiHywGVtVVimECrz13Qu8llLujdXjJ5/yOXDqyAkwCvgaDtdD5vkPkQzTmrQ4YOR6KyGouaW7Hvqadg1De+BoSD5DGeo7se0ZmCBDvSGcybNAnvPP0Mpr/1FprbVmDAkKGorqyysjzSGEUxJQkSdC5HF8jdJDECiqB2FxkQhZBC4vJwRVa1n7IZ5fxKepQV14yigSPbI4C7lEjOrsCuWUp2i84q/RL+3kGDBqO8qhqzm5tx7NlnYtCGo5ENBgFfAAFrm2fDHuaxmm5TeAsc6D4VnGVHJoOF06fhjUefxOeTpmDe4nloGDQI9XX15pwqxdeNUoovC3AK9vAiuWkEogyiuwKyJEGBT1RE4OOzG2hSgYibEKagldQW1+HVeTQwNCu5x3cDUYqwasHgQYMHo6SsEiuQxh5HHobRm22OdJCt+bwlc3xIewvNBpMAACAASURBVFY+B/hCW85D960gwb5k9iy8+eiTWDjjQ8z66EOUVlWjvrbOdHb1aNcFkFqiKCcBqCanBL/6tktFEWUQwN1MSOWZC8xSSvjM97Qqh6y766y60VZuT64ukOs76jiufi+LrxmBdEj+g7oR0F+prahB5YBGLE534Ts7bIcd99oD/njc1lNVwpiftMk0ycJSawoW7NlMBis+/QRvPv4UFk2fgVmzZ8AfjmLo0KEGdPL2la1LKodUlpyWVqtgi87I8eSz+DYBKa4ukIkGqf2G/ALlshPYbmZld6C7M0P32UHbamoWpZFfIIqmZqv8DkyPiCcSqK6qRsOgwWjt6kJVQz222nMsNtxsU/iiUQM9nVbKk4UG9vyMW3AOajaD9vnzDezLZ8/BlCkfIJkFRjHnu6bGgkqc3mUtpYgI0LK6BL10dz2Lm8tiK2lLlkOWW/TETSZz1ROlJgjIcjg1u7gVT6I1ojlyjt2gkvZzuTsHtOiMWfugDxWJUlSVV6GuvhEVdbWYvWAefrjLLthm773hi3n9Ir1lawpArej2EwrSQeWPal+yCG8+9Dg6583HxMnvo7WtA2PGjLGVK5QuIIogsEv3lhKjHBlup84D4tECuetE8jgq8pBTKQutgJAokBu0cgNbojWiQ/pu3QeNBomOpwHgOq4qJFGrv1DQj0gogng0hnhpKWoa61HX2ICFy5rwg912xxZjdwUiYcugCTAXvsDwXlBg/0JBzaKtaRnefeBxpBYswnvTJmLZsiZsOGoU6urrTI1hpFFOowt2gtAt5JDFZAqB8l9kofmZq5QIVHrfBTr3JX+WY+n6B919BwGYx5OfoMGlCKsoi+vEKhgl7Z/nchUhzQTWNzIeR6K0FHUD6jGwbiA+WrwUu510HL7xwy3ZmwBBWzm7sOBesGBvX9GEiY88hY7P52La7BmYP38hRgwfhsGDBxmFcWmM8k9IJdx2Gsp8FHhVWSQn0eXO3Z1WvnYdTKk94tkaUHJyJYG6PFyUSA6wvocGp6vFy1cQHdIgkHWXkVaZnhzXsvJyjBo2AoFEAs0lURz9q7NRWlVjeTRFsK8TU1sW7SuWY8oTz6Llo0/w8YLPMHvWHAxsbMDIUSMtgspGSQKNQCutXfIj+z6qyJrgkEKjFAHRHjmhArQaovI8rnau8/ASupxdM5IGnay/LHN3RUYzizuT6LaIs4vny1kVLZIvwO3ptEZCUeu40Dh4INp8wHb7H4DNtt0WvghX8igs615Qlv2LcZhFV8sKTH3qeQP73KXzMX36TOtwu8km3zI1hjTGVUMEXFdyVLcuAkcDQeARfXGzFOXgikZwWwFSAJW1FOik7riF1JIOXYXHPSZ/p9QcOdHKoCTd4iBVYhmPL0dVqpGOz3OGA1FESqIYMrgB5RWVyNbU4biLfgtEIlZTW0gPm30LSY3xbk4WXW0tmD7+BbR+9DGa2lswZcpULFm0yCz7sGHDrFpJtEA6NcHqKjGu3u6qHQS4q56oOxetP+kRwcX3CFY+ZFVlqcXdBXQNAM4EGkSu0kJwihIJqK6DqvOIx/OZv2PZsmWYP38+5s6diyVLluQT2XgMlRYGAzEkKkowsKEKjbX1mNPSjrNuuA5l9Q2e9i7evo4njRWkzi6wJzvbMPW5l9AyczY62prx8aefYvr0Geacfu1rX/PaPYdCBnhZRYFdVlyKifLW5ezJYhNk6q7rSnyuoyigC2ACvAaBqMLKKEP3z7q3xfjCIf9yP3hxfZ5DoOa2tPrsibNw4UIbCPxb3tJsBerVpWWobqjD583LceJvL8SAjb9pncXy6QP8l8WZvuy05lJ37LLn/dls/5Mu5QsVnGW3/o+pLsyY8DKac2Cfu2ABJk2chGSyC9/4xjesiIMWmABX8MilBAKKgCsLJ/DoNQeMLK8srEDpWnRebDmL2td1AN2op6iSrLtAr+/iyp/aVpKjLJjrkAr8Wv9VaQv2GyMhZLqSaFnWhKa2Frz/4TTsdcTh2Gjrrb3GJOwK7PMhm/UhspIV+FgE4g5g9zv3JwpUsJadlz+dTmLmX1/F8inTkEl2YeGixZg86QM0N6+wSGpjY6Pp7U1NTZYOoPC+AOGCXUB0QS1LzYuo1ewEXlkRDQTXArvWWe+7dIYZi1zike+59ESAl2qj2cUdMDqvlCHd4O7UR6uHGDDZdSDL5cZ88AWCSLGFYCSMcEUlomVliLMLcnkZYuXlCEZjXmoBTbwNAOsqa8aedbDGdPqxXFmQDiovOvupzH39Lcx76x0kO9qworkVU6dMwsKF8y0/hq2r6ahOnDgx3/Oc4BRABSY6sgq7qwuXu52rd8viyrrJksvqCnTuQOJ5+LkcVJd3uwNDAOX23Z1d97jdUwbcqC2/P/+k2NisQIga7XDoCVPds0wNA1Is8ggFkWSuTnU5ahsb0TB0KKLlFUZpOEA84HN5m/7dr6MgHVSCvSuTRtOkaZj92j/gSyXRvKIZ06dPxWeffYJojKVr1Rg8eDDee+89cyrV81yyJJ9psQVwSXmulXcVEtGJ/ybXCagusFyKomnfpTHdLaV7DHc7URwdQ7OGOzjcQcHt5KBb5zCzzn4vL8bQn4U/EEQ6nUU641GVVDaNLtYLRCJm9asaGlA2dAgqa2sRCAWtL3zWBk3/1OgLyrLnaQHrStMZLPvkI0x57kXEO5Po7OrAlKlTsGTZEixvXoG6mloMHDAQ06ZOtZvEiCJrVIcMHAQGWqJxb3WL7oBy+Wl3NcWlMXJApa3LSov+uKqLy68Ffu4nBab74OBnHISqYOLn4uVKN3C/uzsA3UGp3+IGx0zuzGaQ8nu5+wbyVNoGgT+ZQoo+TiqNzq4UItEokrEI4tUVGLDhaIz85iZAJG5cP6Ce2f2IuBck2Hl9edPbFi3CO0+OR6K9E53JDrw/8X2sWLECcxfMN+lx5IiRmDVzJuYtXIChQ4Zg9KjRqKvyMiLDMY++uLRC4OjuiIq2rMyqCqguveB7mhX0vmiMzqH3RTlczLh0SUAWiPOqQ45auJTHbeSkwScfQM9eslkKSa4Wnlv4zCw9jT2LV1J8374lF2+yUo9EVQWyZaXYeNttUDVyFLK2RGU/QnnuqxQu2JFFqqkJbzz2BOKtHWhvb8HkKVOwYO48A3uirBRDhgxBKp3GhzNmYPjw4RjCip5EqfF29mDRku+8VgKj2+2LgFG4XwNAYJMz60YyNQgFIllf17J2pzI8niy5gkwu99b5NMtoxuAg8ax9Bhnrgem11HNnKneQKvnNC6B12hqyytzUwJQjHgpGDPB8XcZOwpEwghXlqNpoDIZ+59v8oF86qgUNdrS34a2nxiO0dAW6Otswe/ZszP5wJubOm4dQNIya+npMnTYVjfUN1ta6JBZHIubxd1p2cnnp6KINinyujCO7qbcaIOLGrtUX3ZLjq3QAWWwFrOSUasDk5bOck9p90MjZVbsPRUz57DZxYnRVg1eDRZTFBkgmjYA5qR5/zye8Wbkeu4uRQhHQfoQisOZT0UQZyoYNw6itfmjt9/pTbaurehWczm4Ay2bg6+zABxNeROrzBUh2tGLBvAWYMW0aPvvsM7R3dSFWVoL3P5iIhpo6DB40CBXlFQjxBoZCKK0oz7fJExWhMmNWn+2icxmMrmIiysDzu9VLGgQCI7fjMVRAIqmQ+5FGaCApr0YWWIDUsfls6grD4Lkek7yxSjXWQHPTjnlsUSOBWDPUF7MUfRVvePIzfU8CnM5nKpkytSYai8EXySDBLsLl1YgPHIwR2/4IPr7fjwq5Xem3IMFuwMsk8dnb72D+e5PgSyaxaPFCTJ00GZ988gkWL12KYCSETz/9DMMGD7E8d16UaDhilp3OF8GtthsEDF8rFUBW2XPgPHogMLuOn2vZZbnF2QkkRWddCVNUhEAWAAV8VwFSuq8sub4T9+F22t9VfDSQ+J7ydhT8cilTJus5p9w+FAojFAoinWLnAo+6hUNR6wsfjPlRGStBIl6GSEMDhmy1JbIltOz9K68mPysWXm4MTFHIZpJWqTT7b68j09KC5tZmfPDBRMyZMwcff/yxgXfp0qUYNmSoOazi1FI3SGG4DQu0ZcEJdgGJz9xGOef8d3eHUYAUJRHgxfG1vVuALdCJy7sRUFllafikJDwGKZfr9GpAST51B4tmJff48jHycmRuFUIdR9ZddI7fl5Y9Vh5HebQEiZJyRBobMHTrHyAbjSLQz5qoFjTYufAtwd61aDGmTvgrfMua0dq+Au99MBEffvih8Xda7daWFpMgGU11ubGme02BcgoFdC2vLifTtcYEiEDmqikCuMvf5Thyez5cn4AAtaVkzNH06Ikojd7jzKBYgL6bjsl9lP/jOtOSPzUDiLe76QRycHV+Obb6flp4OJyIIRJgAlwpSocNxbAfbYks4xP9iMZ86XoXmmW3KLb14s4g1dqKSS++hPSn8y2SOmn6FEybNg1Tp041sFNKq62pzS9QIKdOyodSf2VtadFcCiPrr7I7zgKcDTQ7aEbgcTUAXJ7vgkqKiiva6fvo/C7dkZQo8Cr7UsAUp+dr+RMaJLJ08hfc3ytaIydWA1G0hs8cBObDBEOIsQc8+98PH4phW24JlMRySWPuL/nq/22/tdDAnr+sGSoJSXw08X0seut9BLo6MG3GdEyfPt3SBJQaQJ7OtniiAaIcsoZSM2hFxcdlhWXh9ZpAMZ0+F33VjEBwScoUwLvLgAKiO6uIRsgfcJ0t/VtUSDOHwOoOFPkO3c+hmULWXZZbKcqy9uL47uxka8lmYP4N89/rxozByO99D75YpF/q7AULdlPN6KMijUx7Kz5//W0s/HAGPpkzG++/+y5mzpxpbZ7j8RJ0tLVhww03zHN2trZmzgdTPaz7V8pbP8n+nUlbc1A+CGo9ZO0Ffjd/xqVAsuqytnymhUymktadi6DjcaVxSyMP5PJOxPltIHYlLUyvY/r9XBvVy1MRvQoEA/kilSBX6GAnsJxaxPNqppCT7YE9lzqQi9LyPS2SHAxx0TKfnZfX+LOlS6wtx5bbbYvhm2yCSH295QKH+2FCWEGC3RLB7JZ4PVB8mSxSHR34+O13MOW1V/HGCy+gdflyzF2yBImKSqSTSVTV1FigieJy2BdEOpfJl0p2IZ1KItnVgZb2Dhsgxu19Pm95l1yRhni6KAUBQpokoBvF8HlFGK4Tm0ynEAyH7JhfqDTs3+JlPvL7cBCEggEvhM/zJ1MI+gNIdnXZoPRZkYgPAZNEg7CBkUlbkheTs9jzyOf3WWYjO4Ax0KTkLT9Xw2ZaBCXJVCo323mR0SyLPKjCAOjo6sKiJcvw+YIFmLtkKZo7O+CLRNDSlYI/HMbdD9yPBFchDPJ7e90J+sujoKVHgj2TA7u1ZSZmuKz6imbc9rvLMW/yFLQsXoKFC5egsq4O/lgUAzYYjm9v+T28/vd/oH1pE+KdaSvj4z3r6Gq3qGJrs7c+qgWBqOPnKogEUiWTSYvXuk2y+uGAl36gASDrLqogwJuuz6Qqk/58CPi8NU+TmS6bVfgxLX5nR4fNXrLYjPrasQn2NPNngvD5aYn9tn0gzBmLyyITjVxUjMfibBCw6D8HFSlWS0szFixehDmffoJ5ixdiwbJlWLp8OZpSSfhDYQRCEUS5GFtDAyL8Tdks7n/oQVRwYTYe1+sW2V+w7hmNXApJQXL27tyWrz/56CMcfsDPMLymGjFa/BSwcMlyzG9aimvuuhXf2GwTdLZ34ONpH2L2u+9g9pSpaF68BMGuFNIdHWhpa8aK5mYvQYq6OleyyJW4idaIq/NZ4fW8tad1z+XbhMMhLxjEBCsCg8UduVbSTGIjoC1QFAx5oPRsrZeTQiuczYCzQsgfQjgURjgaseORXnSkupAN+REMRxGOxBEKx5AoLUOsNIZQNIJoaYmX+xOL2oAghWEV04qmJixbthwtzc0Y/9RT+GDKVGyzw3YYOWYMOlMpvPzqa3j9jTcQ8IeQSJRZMl2IoVZfFvfedx9q6+ttBuFX7E9gl19i/lYhOqjitu4PfXL8szjvnHPRtnQBsqQAaT8CwRAq62ox/sXnLWpqQRf2g0l3ItPegfdfeQ1vvvQK2hYvQUvzMixZvAhtzS0GUi7JaPw4SOvoURTybVphrrXKZ34uqkPQqjpKfJnUg7RCtpBgMbDTIjNHnPnuuSVn2HW3oyuJUCxi65pmqK+XlNjiaKF41GgYl3Yvra5EtKoc5eWVCMViBnZSnSyblwYD1qPdxpflowfyNpjW35ZOTmfQusIDfl1jYy6CCvz9tX/gmKOORntrG0pKEraKSSgSRGdXJ+6++27LNbJZyTql9h/L7k4xhQn23C+0deSyWWRSaVx04eV44onHsaJpCTq6Omx6D4Uj+NG2P8JtN9/q3SOb5jMGQBIJfyqNjtZWfMa8mrffwruv/xMfz5yFVEs7or6AcfhIzJPg6AwSzCXxEuPOVCk4C5Am0MqzKoirYngg9qMr2WX53z7yeLPeQIx5JrE4fIkyRONxLF6yBH979VWvmiqZNl+ktbMDPxm7Kw4+fJwteUmnkd+bHNua8HJ1DX8glwBG+s/uvN7AyRsBFY+aHu4BU4UcFpDz5RLIOLv4g2D/zMmTJmO//fdDc3OLBZQI9pKSuFV73XHHHdhowzFFsH/V5I3TNJWU4487AW+/9Taam5uQSiVtKfRwJIKzzv4VDjn44Hy+i6zSF7YpayDJppLoaGrCX8c/ixefeBJo7UBL03KEwp7TySgm+9GEI1Gz9GFWOUVCCITD5oSGQhGE41GUlCZQVVuDaEkcFbW1SFTVmCITj8cQpGTJNVoDXvewCRMm4PDDD8/B0Ycwge33Y9/99sMFF17wRSlcN0vq2tWeNAbwWO6Xy6s/nDETu4/d3Yq2CfaammrEY1F7fcMNN2CTTTYpgv2rBjuBOm/ePIw79DB88vEnaG1tRoaZfUFvdblbb7sdm266aR7sNhV3e1gEk/Igs/7SaSxfuAjPPv447r7zTrS2tZrjWVVVjZjd/BamemPgkCH4+bhD8c3NNjW6FIjSuaMV92o4c2mF1iLaFBrKhh7h9YpDAfz973/HwQcf7OXfZL1gDmnRjjvuiKuuvtocWK/SaM3ThjmzPsLYsWMtxYIDm2WNJSUxLF++HNdcey2+t8UWRbB/1WAnUCZPnowjDz8Sy5c3oaOjzSZtgn3EyJG4884/WQG2KwmuDOzMLfM0aB8oST799FM4+6yz0dWVtFycATl+yxYVO+y4I84571ybOciL6VB6vJzr+njSHB1Toww51Ydc2pQd8M8D+zvvvIP99tvPHEhSE0mc3//+93HzzTeb3GgUaC2Afd7n87DbbmOtFw1nIqZYlJUlrCXHRRddhB122KEI9q8K7IoK0uo++OCDuPzSy83qdnV1eBJd0IfvfPe7uOmmW0wTd6uFun9nLyDh8Wqb4n1ZPPXkUzj77F+ho7PTjDR70dCy09Jdeukl2Ha77Wx0+K020ytiFjXIiRg5haX7NPIFf2Bqw2677WYNjqwLQE7X/9a3voX77rvP/IS1ZdmXLFqCn/50V0uRpg/CVUwqKsqMs//yl7+0QVl0UL8itAvsdBJPPfVUTHh+Atra2o2vh0JcbQI46KCD8Ztzzs0HdP7bV6WebLq9eXNZPDN+PM4++2y0tXfYW7W1dYhGI1i6dBluvvWPRo2kwXsg//e0Vx0uN37yzCZX+WzAosWkZXfBzojvk08+6U01xmTWPI1ZtnQ5xu42Fh999JENOmaKEux0ng899FAceeSRRbB/FViXzk6LyyDJHnvsic8//9xAQ2WBagkpxE033YTtt/em3/8FGDUE8nS7LP7yl7/gzDPORHt7hzmwdXW1iESiWLpsKW659SZstulmxqm/OO7KAOm85yI/NwUsWrQI22yzjTmB2bSXxRgMhjBw4AA899xzps2vSbC7Em5z0wrstddemDFjpilMLHYpLStBZ2cH9thjDzMoRcv+FaD9i6gZMGnSJBxyyCFoa/O68vKGkMawFR4BQ/qxKmB3fwaP//zzz+PUU09DRwdpTNaOQ+mRNObmm2/E5ptvvtrH7X6pCHKCnb0a00lviXdaVTqHL7zwAuIlsTUOdht3Ph/aWlqx//77Y+LESWCagcBOWrjtttviwgsvLIL9K8C6EyIG7rrrLlx77bVYscKTHMXNN9tsM9x77735HPL/Zdnd30EO//LLLxtX7ejosvOpOzA57I033oBvf/vbvQY7E9BIY1hdlUl9EaCixPniiy+iorJ8jTqobmZlV0en0ZV//ON1s+zl5RXmoBLspGx/+MMfimD/KsDu0WpW5mdwxhlnmF5NOsM2EcpNOfbYY3HCCSfkswZXB+w89l//+leceOKJaG1tt2NwvSaqFLTsf/zj9fjOd75jP93NX1/da8FBtffee+Pdd981y64UYg7YFya8YCuJGG1fC5ydkdVjjzkGzz33ggXFShNlqKouNxozYsQIi6IWaczq3uE+2p5AodR45JFH4YMPPkBnp1fCRsAQlFdffbVRBDftdlVPTbC/+uqrOO64442zC+yiMTfccB2++93v9tqy8zccc8wxRplcy06wP/vssxg0ZGCvz7Gqv5mpzmedeSYeeugRK7zmSuHV1RU2W3JWe+yxx4pgX9WL2ZfbKc9jzpyPbepdsGAB2ttb89Idb86f/vQnjBw5ssdgZ8Dn6KOPQWen1xFAS07Ssl9//R+wRS7I0hury0FFLkwqlupKm2NNks7zjR//tPWbX1s6ezqZwiWXXILbbrvDZNSy0jKUlZfYzEJfgrOnGY5ibkxfQvl/HyudZn4LjGpQJaCj5/F1r7nnBhtsYACifNa9NvR/H92jSK+//jqOOOJICyrxIc4usJPGqPJnVY65sm14Hn5PAj7Z2ZUfrATVQw89hG9svPFac1AJ9uuvvx5XX32tNUmiZa+sLLNoNB8vvfSS5ekoqtvT37wm9yvIRDCBnVTl9ttvNxUmk0lZMIQPhtuvvPLK/xpI+m8XnfSCYCdFomUX2Elj6KDKsvdkIK3MEaaGTbC59aZMvtrie1us0aCS66Dy/AxknXvu+WZImIRWXVNp1QO8vi++9BJKEwnv+/TH/neFmuLLZpy8IZTKmCrgtbvI6euZDM4991wccMABqxRM+k8W97XXXsOxxx5nYCcoGD6nL8B+kn/4wzX43ve+16NZozvYp0yZgj333BNUQ/iQmsQYwdbbbLNGLfuXvksqbbGFE044yRx/5sfUGNizNnO+MGECqnMFHL2hbkXLvppXgEDncio77bSzRfi8Tls+47y0jnSmuOJ1Ty0vwf23v/0Nv/jFCXmd3QX7tddeDeavqBZ0Nb9+fnPOIFwTaeedd8aK5U02OFX5xFnr/3baaa2CnX7KoYce5oE9FkdVdYXV6nKAP/XUU17hOquV1oI61JNrWpA0hjfjr3+lDn6yrRznVfSzS5bfigyeeOKJfMuLnlihtQl2Jlox2/DjOR/Z4BQVu/jii7H7nnusNTWGNQEM0O2xx16WKx+NxlBVVW7XlN+R+Uf0hYpg78kw7MU+VC6YY33bbbeZZSc4meVIpYChbWbpqa1ET8H+yiuvmE7f3u7RCyZGMaGMU/pVV/0eP/jBD/rEsvN4TLKaMW26pRKr8xip2H4H7G/n7slvWN3LS87OTmo77rgTurpS9lurqioQDHpgv+eee2y9qiLYV/fK9nL7ro4unHzyKRbl1MrU/qBXFkf5jLRgXQA7BylnJqY7vPPW2wZ2dek67bTTcOi4cWuNxhDszNXZdtvt0dbWYXlAVGPC4aDRGBoX+ileHeqaT0zrCUQKksYsXbzUNHAGk9Q81B/0WwPTW2+9FRtttFGfgJ2cnUElWtY1YdkJdjrXnEEmPP9C3rLTF2D09qhjjl5rNCabztiCwj/84VZoalqBcCiCispSRCJhe/+yyy7D9ttv36/XVioYsEsm44j/9OPPMG7cOHz66af5Zv5M6d1wzIZGbRja783UTwsrNYZpw5wlBHZaOdGY3ursPA8HK1OJH3/0sS9Z9qOPPhonnHSiGbjepCSsqoWkZed32WqrbbB48VKbYSoqSi2tmXIrYwE//elPi0GlVb2gvd1OOexvvfG2hdkZ4OF71qQoFMCuu+2K3/72t70O9qwM7AxQkccK7D/60Y96rPboOvC7E2B0Ru+9+578wCVvP+igg3Dm2WetNbDTQaWjv912O+Czz+baNS0vL0U87smtZ511lqUA28Ar6uy9hfJ/319NhgiQe+++D5dffrk5p3m5LujH7353Of7v//4v3waup9+I58inC7R32jkqKisQi8awvGk5rrzq91/Ku+npefib+Ec+fM1VV+c7DRPsBNYFF1641jg7wc7HrruOxeTJU6xvO7MeWSjO63zCCSfi4IMP8mZMr6qw3z0KisaIyvzyxJMt35vOKakErVBpeam10uAaqL2d9pUucOQRR6Kzw4ugyrJzSr/iyt9hO5bl9VIpse5j6TTuv/9+nH/ueV8CO53sK35/xRqNoLpoFdgPOugQS/NlJ7KSRByJRInNPkcccYR1QrBikiLY1/xAJzCoXuy5+15WPsaboIKHzb+zOW6//bYvdfHq6TciCN9++22MG3cYOnPSI9tVM6pIqfCy311qYF/dopDu34eDir+JWY+/OO74PNipKm211Va4/oYb1loiGMHOYqrjj/sFnn/+Bct8JNBLS1mt1GmK0XHHHeu17WORbT98FIxlV0daFjrsvtseBnqCXUvDHPeL43DUUUf2CcclCLlg8MEHH/IfwU5loi8sO4/xr3/9CwcfeFCu6ZK34gezKm+97ba1BnaqMRx45513Ae6//wGrPE+UEuws4OjCvvvtixN+cYL10elHrR6/NOQKBuxyTmkFT/nlqfnlX0hh2I7uD9ddi+9u4eWY9wWN4YIG++yzL6jp8+Fa9ksuYIq3QwAADwhJREFUuzjfWqI3qg9/EwcxVwsZu+tu+QXGCHY2Jbr73nt6PXusqgE2y57N4qqrrsENN9xoBRyJRDwPdvoQJ598sgkBRbCv6lXt4Xbit1dddRXuuuNudHR4xRqkMQ0NDfjTPXd5/QktDbV3pJI3fdasWdYhS5x9TYCdl4J9bxjM2XGHHxtF4m/ibPX1r38dDzz4gOnavRlQq3q5WajOaiXms1/xu99bAhhbh5SWlVp3Y7b8OOPMMy19oAj2Vb2qPdyOYCd1YeT0tVf+gXYDO1e8CGGzzTbFLbfeYk2Lepucxa9HsFPD32WXn6Kjzesu4Ors5OyiMb0dWKQOVDu22WprC8vzXMyuHDNmDB546EEbvGsD7FzFhI8HH3gYF557gQE8VhJForTU6M0uu+xi8QA/m6UWpcceongVdyMI2JrtqKOOwgfvTUEqzfxvLrgcwrHHHoNjjj0mH8buLQB5LrbU23mnndHW2m4AZLcCFkIzmnj5FZdZxX1fOKhyUn+y085GZ3hM0hhmbT70yMP5hLZVvEw93oz1AHw8+8xzOP2U040mRmJhlJaV2e/faaed8Jvf/MabaYpg7/F1XqUdaV3YG+bAAw/C3M8W2DTLJCWm9d5zz934xjc3zlvA3lpCziJsb7HD9jvkwc7KHfoGBPtV11yJH/7wh33iDGsm+dn+B1jBCB8E+9ChQ/Ho449ZIKu3g3dVLnA2tzbqKy//Dccfc3we7LTsfHAmO++883K9bIpqzKpc0x5vQ7C/+eabVj3U2swiaOZ++62hEPsysrW0Hn0Bdurp22+3PVqavcamLtiv+cPV2HLLLXtt2fV9aTlPO+VUPP7440YZSF2YqvzIY4/aedcm2N9+8x0cMe4Io1bhaMhoDL8fpdYLLrigCPYeI3g1dqQjxz4wl112OTraPH2dNGb33cfioot+m1tWpW8sDm8uLfh2222PpmVN/wb2a6+7xoo3ektjXLDfcN31VkrIgUWFafDgwXjo4YdRWVW5VsE+bcp0HHLQz7F82TKEoiEbbLweW2+9NS66+GIvFaNIY1YDuauxqS3olVtm/KSTTrIqdzeYxNz1n/zkJz2uN13ZV9H6qD/e4cdYMH+h3WzedHJ2KiZ/vOkG6xvTF86waMxjjzyKU045Jd8OhGD/84MP5DuarcYl6/Gm/J2MY+y7775YwiV4AiHzVfg+8/cvv/yyXGfhHp9ije64zuvsAjunVSoCbAaqqZ4t6VirSWdORQ99cTV5TqoRP9n5J/jk40/zYCd/piJ00y03WpesvgT7G6//y+pm+dv4W9hmmw6qMjh7S81W5boQ1Cx33H333a09SSgYRnlZuf1+5rL//vdXFMG+Kheyp9soAYxLtLN8jSqBlkJnmdidd95psmBfAU+WlrRpt113w8wPZ+XBTkmQ57/ltpvBttJ9SWPmzJptiodmLcYMSGMaGhvWivSo382Zi9VetPB+X8DAzgfb/V111ZW2ykg/rd1Y9xcQU5rA+PHjcfrppxvQJc8xv5p51u76oz0dVO5+kgP33nsfTP5gsoGdFIZgJxhvv/M2fPOb3+wzEPL4Cyh17vwTk1f5exgo+/MDD2DAwAFrhbPz9/NaM7mOMwy7NvjhNYglT2dE95prrkYoHC4mgvUFyP4Tf+b7TOmlg8q21LTiKsEjtZFT11ffgcejZT/wZwfivXfft+NTdhTY77r7Totw8tEX9IJgJ0fefexYs6gEOy07wT54yOC1CnbSKGY3MsXZl/VbmgTFANafXnfdH4pg7yuQ/dtxuKAvrU1nJ3550knW3qIrmbQVKWhp2ZKanbr46Et5Tnk4hxx8CP71+hv/Bva77/0T/t//+399CvblS5fhZz/7mVX4y7IzN2b48OF9+tv+073Sb+bzmWee6fV2hN9oDMHO33vDDdcjHKFl7xvVq69xs247qFlvamWlzLhDDzUg0JJyRRdmBbIET6VxfWFhdfF14w8//Ai89rfX8tKj1jm99/57wNUx+tKytza3WN9KxhL4m+h8333P3Rg5atRaAbtojGZRXltadqpQnNFGjx6Nm266EZFopJgb09ejVMdjNh4bCZFHUomxErxwyIqUOd32tg50Zd9bYD/2mOPw0osvGdjJXQX2Pz94vzVN7UuwczGAX/ziF9aXXWD/0913Y/QGo9ca2PW72X/y0ksvtc7Cklw5w9xyy81FsK8poPO4LARm/3ICm0oBwc61RrkAQV+0oPtPYOf7J//yZDz7l+fMKeZNp/RIB+6Rxx7GsGHD+oSvy6KysSmt6RVXXGFgJ2248eab+qTyanXuDwc2q8BoTFLJtNEYSqEc3OzcEItHi5Z9dS7oKm+bBdIpr+Emg0cEHS98XUO9Ne2xdmy9TOf9b2DnmkpPPvGUnZcOKiuVKD0+9sSjGDRoUK+lR1pSPVTdz36L1Lp3GzvWFiNQC7++pGn/7frzO7FwhYElpsvwd3OQM32BzVajsWhRjVllAK/GhjatpjM2vdPa8DUt+6abb4ZbbrnFgM/Xff3QdM6uXA8/+DCSyTQSJQnE4jEkkx147InHbaD1hc7Oc/E4XAyAyW3mk2TpcOcWJ3OXae/rH7qS49Gye+nNu6CjrTO/sjcH95133WkF2MV89j68EXmLxyZCHZ348Y9/bCm34si/POVkKwBWi+c+PLUdijecj4svvgj333s/ujoziMXiKElEkUy144knnzYdvC8DWTovf3tPVgvpq2vA81MQYApz07IVebAPGDDAFnjgomZFNaavrnaueEKHmz1zllkZ6t4EAa35Pffdazp3X5TgrexrK5B1xRW/w1133IVkEohGWMgQQyrdkQd7X1j2PrxsfXIogp2BM4J9wbyFRmEo87Jrw3333YtYSdxbkKAfPtZZ6VHW9ZGHHrbUUks5DYeNO47/yzPGZdcEX9c95PkZHr/15luRSgHxWAniJRGkM5148qnxdvM10/TD+96jr6QZlc9Mrpv14SyEwxHj7YxnPPjQgyZDWhPZfvhYp8FOwF12yaXmjNKyE+As/D3/wgv6nEK4907pAjfe+Edcf931SHUB8XiJ0ZhMNoknnnzKIpyFDPYDDzwQb/7rLZNbCXb2pyfYS0riRRrT1wNdfRBZ1MCV49T564rf/x47/2Tnvj7dl46n4u477rjdOnV1dXHZlZjRGPhSePyJpyzoU4hg50Dn72cngb+MfzYPdsYZuM5TWXlpEex9iT5Np7zof/zjH21hK1p2KgJcQ6kvNe6VfW+en+e75+678bvLf4eurqytRCGwP/X0M2bpCg3s/D0CO3tmsv+kWpWwI9qjjz6KkkSiCPa+BLsuOi88gzhcSYN9XBhOp+S3pivuBfaHHnwAF/32ohzYPc4eDME4O9OKJRv29W//Ko/H38S4AvtPsnpKYGdC2MMPP4yycm/V7f74WGc5uy4ms/Bcp3FNO6audXvs0Udw3nnno7MjbQ5qLB5GOOzHU+OfWWu1oWsbVPJXuKL15ZdeZr4ROTv/Hn7kEet5af0e+2FS+zoP9rV9s3m+fA7900/j17/+NdrbkiiJM6gURiQaxNPjnzH9uVClRxqYJ598Er8662z7jZQemS7BdZWqa6rXWrPV1b33RbCv7hXL8Vbe8Beefx6nn3Y6OjrS5qCSxpSVx43GqAywP1q4HvzkL82etO5c5PekE040qibLzrQNBtOYddoff3cR7D2483KQJ0x4Aaefejqam9vzlr28ogR0UOk3FKKDqpmNxRvHHn2c8Xfyderrf/7z/V6ZYJGz9wBV/XQXBbRee+1VnHTCSWhp9hbUos5eW1uJRx9/Ip+T0x8tXG8uq9SYiRMnYtzPDzOBgJSNf+wjP3DQwGIiWG8ucH/cl9Ljm2++geOPPR4tLZ2IhCOIxkIYMnQgHnjwoa80f2VNXy8CfsaMGdh3n/3Q1dllVp1gZ3Bv2PChxUSwNX0D1ubx5aC+9+471oFsRVO7cXaCffiIwfjzAw/lv04hWnaCnYUyXPSBNQQEOgFPsA8fMRzwedmZ/e1R5Ow9uCOayidPmoRxh45D0/JWW/GZNGbkqKG45977CxrsHOyLFy82sLOdNtUYpg0w63HU6JFF6bEHmOrXu/CGT582FQcfdAiWLWuxCCqlx699fUPcetsdeee0P1q43l5YDnb2utxzj73w6aefGNipPrFcb4MNN+i3kmvRsvfwzhPss2bNtOVflixeYfns1Ng32/ybuN5WpvCm8UIEO2VXtizZe++9bVEGgp3BJQaauKByf40vFMHeC7B//NFH+NkBP8OiRcvzlv173/82rrzqmoIEuS6V2v+dccYZtrgZZVZmebL7GtvyFcHeQ1D11914w+fPn4d9994HCxYsMwc1HAlgx//bHhf+9qKCBzt//zvvvGMlkQQ7uxaff/75a21xhJ7gomjZe3LVcikDixYtxD577YN58xYb2CPREHbdbSf86tfnFDTYdckYUGKHMj7TsqsVXn+lbkWw9wLsS5cuwd577o3PP19gYI/FI9hzr91w6mlnFDTY3RRrN7NT9KUI9h6Cqj/uppvNBb322Wcfs26MoHL1OFbwcGrvrze8P17PtfWdipa9B1daYGdAhYrEnDlzTGdm8fFhhx2GI488sgj2HlzXNb1LEew9vMJ00NgQac8998TMmTNNZybYjz76aIwbN64I9h5e1zW5WxHsPby6kt/2228/61XOih2GzNkW7pBDDimCvYfXdU3uVgR7D6+uiq73339/vP3225bTTcCfeOKJRbD38Jqu6d2KYO/hFVYyGHuVP/3009bGg4A/55xzsOOOO9rrQqxB7eHl6he7FcHew9sgsHPV6YMOOsi6ZKmTLYsZimDv4YVdg7sVwd7Di0uwU14kyJkfwsQorsrHguO1UfTdw6+9Xu9WBHsvb7/bEo6H6q95Ib38mQWxexHsfXAb812Fc8cqBpT64KKugUMUwd7HF7XolPbxBe3DwxXB3ocXs3io/n0FimDv3/en+O368AoUwd6HF7N4qP59BXoNdjln67tT5jqphXgtCuE+rzbYuztghX6Tu9uqlTmg64Mas7LfqGuxrgyE1QK7WkgwaMKgCots1R1LP7yQdWZ1sO2+gJeuQX8vXugNydC91zHcgnJ1Ul4TCyz35jt33/f/A3lb7IWxiW9BAAAAAElFTkSuQmCC">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -410,7 +407,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1035" name="AutoShape 11" descr="data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAALkAAACLCAYAAAA9Hzj6AAAgAElEQVR4Xmx9CZhdVZX1usObp5rnTCQkgSQkEEBmlVGRQUFRnG3axu62pf3bEbUdsdV2Fgf8UXGeAEVFEZAhjAECSUgCJCFjpSqp1Pzm6d7/W3uf86rwt74vXyWVV+/de+4+e6+99tr7OH/97vXhRKmChatfhkYQYuzoFKq1EprNEImYj0TEx/TMLDq7ujBbKOI/v/4VLFq/Cv3HrUDP4ELU6zVUSkU4QR212TwmpiYR7VuCdDyNTCaFnu4+PPHgXTjj9LMQyQ1geHICSzr74DabKD2/E0///g/46Ec/iqVLlyKdyWDDgw9i4ZIh1Mp1PLxtD3LHnQg3dBACKJVLKM7m0d3dDdd14fBPs451/W2YKpWxe3QKZ65bhQ1bd8B1gV//+EfYu3M7ENYRhg4ajQaajQCxWAx+LIZ4OolYIg4/lsA7T+zC4u4MugeGUAvqKJfKWHTsiUjm+uF5LpphiGaziTDklQBB0JR/+34EYbOJIAgAhPL/vu+h3mgAYSif6XoewrAJ3/Xkuhv1OoqlEjzXhec7fJn8XjQaRa1Wk/etlsvwPA/NZkM+3/d9eU2j0ZR/RyJR+cxm0ITnQj6HV8b3b8p9NuF7nryGv8fv0VgE9Xpd/u44+jvRSBRNXnsYynXm83mkUklUKmU4joN0Oq3r1mzK7yYSCfkMXk+lUpF75b/5f/ZzAEd+l/cSiUTgOY68lvfDn5fLZWSzObkGXksQcN0CubdEIq731WzKOuv7VBCPx+XfsvrmWvmMItEIgmYTjuPK/zZqdbkffm5o3sd5y1uuCPs7snjzVW+A6/nwIwlEkmmcc955eOXZp+OUNcejUi5iwcKFiERjuPZzn8Xa885AYmgA/YsWwwFQnJ2F5wQYHx5GpVZDbsEypJJZRONxRPwIHrvvzzj7rHPQObgSR6sllItleLUaGhufxYJkHCeccALuv+8+/O9Xv4LCzCwuvvQ1WHXyyXhhdArv/fj/ACE/RRcEQSCLxQfCBYj5HlKVGUyXq6i6UZy0ahme3LYTIQI88cB9eOiBu+GhiWYAWbigGcLnwkcjiCUTSKXT8H0HH3nlQhRLFVTDECesW4uDw4ew+qSz4cU6EIn4cDzXGIcrD52GxofD9+RDdF0PjWZNrpNPQl/jIQjVgPgM6tWaXDPvplKtmg1Bw/TFIPjF35HfazTkPeCEYrRBGCIWjcpD5kOtVmvcUoj4PjzfFcPhtfC9M9ksmrU6LUReW2+oASKkQQVIpVNilJ7nG0MLW5ujVq/L5wTclL7dJLoJueGaTd00spmaDdmYvBYaJ/8vGo1gdjbf2hT8N4JQjI7Gz7XkvXLtqtWKvFcu1yZOgxuB76t2rM6E68ofcROoIesXX8d14uv0D52MI9cua+w46pS4oS964xVhOhrHe666DP39/ZiZnkV7Tx8uuPg1qDebOH7pQpyybjUWDPQhnWvHdZ/7HJadsR5ebyfWvuw0lColVIslOEETB/e8iK5sG6p+FNGOXvgO0JbJ4omH78epJ5+M7mPWolCrYaZYwNGjR9H37IuojE/gTVddga998zv40x9/Jw/l2WeegJdIYvfOnQhXXoAQ9HbcrY54KFpRJOLKQ/YAtLuBLFy+XkMkFsNMqYS4F8HBfS/iVz/6HuA6CJvqHbggfB83QiNPIplOiZdY0RnFm08/RjzUwLHLMPziPixcfiJi6R64UV+8sPUw9gGI9zQPPxaLo1apyrXROKrVKhrGCGRzNgPZmEGzIa/xjGfm6/iZ3AjcEPow9SHJ5wSBGGQk6sva8LX8Nw1KokKjjkaziUQ8jlqtDscJ5L35vnKfZtPRu7lcv6CJeEy9peu5cB1XDYRetdnE0fFxjXT00I4r7xOLx2RDAIH8nJfF9baeWiMaIw2vXz+Q/+Y18jXpZFLex49GxTnYe+Nr+fdCIS+vpxEzKuoG0mjDTaRRUvy6vJ/L5xmGrcjAzy+VihKB7OfyNfw579s584orwngkjg+9+RJ0dnbA96LwEilcfuWVqNbqCBtVrDt+Jc4782USmr/041uQXbYAYSaJNeecDcd3BUJkEwns2bUTC3r6sHN4FO2Lj4ETBBjo68eWjQ/j5HUnoG/pWkyU1Mg9x4W/4wXsuvtv+K/r/gPfvun/4tZbb5WbvudPv8dVb3krpqYn8fvtU6j5UThmx7pBKDueN2S/6pUCGnV96H2dGYxMTiMZiaFcmMZ3vvw5432a4hn5IGlsXiSCqDHyZCKFTq+K/7z0RMRjMQytOBa7t7+AoWVrxcidiCfeSIwRECPjl/XWAknobgJ6OGcODjQbAk0IXcKGblIaAkMsf86Iwt+zmyca8VGtVeV9raE7oUYgj5dA6AGgVq0KXKExibG6aoz0jrF4xHjtUK4zlUy2rpMOgh6Vm4/xRCKFvotEAG4W6wGj5nU0NoE9svkgnpje1cIeenPahb1v/pzGSsehHruJZp2G64Cmyp9zo5TLFbmvWo2bUb1yNptF0OBzqrfWmM6jWCzK/ytYofHyM32BTnbtTQDQe/XVIRD+CKw958rXh64XwweuuhDZTAbZbBtCP4bb//gH/PBHt8jNe16At7z2NWhLJPH7Rx6G09uBiUIBi89Yj5CLUamiu70du59/DoNdPbjnoYdx8kWvRqlYQm9nN0b27sSCrk6sPf2VGJmpoFAtY3psAgsqFbz4l7vwr9e8Cz/91W/wo1t+Jjf+1IYHcP6rX40QTfx0416UYyl4TQ1LXghs2bIV69efpBAmDJEvzshD58JFfMANPUQ9D4kI8KX//pDg6TBQXMmbF1gQjSGWSiKRSiISS6LNqeD6K0+RBzpIT75nPwaWrkE83YMGH65Lj6dGJR7HRAQbKvnziBcxsIPRQkOqPGT+TqC/SwNnHkMDoCHNzs4imUwa7Mz/p6fWTSOwQHApMa+Gdv6hQUdjMbkXPny+nh6SDzUaUzggkM51EeH/1whNNLoIrjdhnJuP3p1Y3WJgXot6Ul0nzQM0v6jVqy2Yxvfjz2m0fC2Nn5tMN57COG4YbqpaRa/d8yMmWjH/iMjr7CbV9fJQKZVMblKX97T5gPX+1qj5vup01HHQyPn7xWJBIhHXjGtP+OW8+uq3h44b4oITV+DUtWvg+XE0PRepbAaXX3KJ/GIQNnD+Oadj6cIBzNYa+MvzW1Cp17Ds9NOQRwNtbW0oFQtIehGEhSIevv8hrL74YoSuh46OLklII/US+oaWAZk2lJohijNTWLNkGR789Gfx6Q9+ALfe8Ufc8MUvi5dmRGD0cBIR/PL+bSikeqA+TBd900OP4vRzzjSOPJQkkQlHJKaelp4p6vtwG01883MfQcBQTE9qIIuE8VgEbjSCdCYnDyrlBnjby7rFmBctWYJatY7B5euQ6RgwiZE+ONkgkhBqAsgHRaPlYltII+EUQSshEq9sjIUPRDwREyPZfIE8CDECwg++r4BQhVd8+GpEUXmYlUpVkkGBSUFdjE+MPhoTjKteNIZ6vSqYXD6Xm4bJsxh3aJI1hSj07rx/xf9AtVJGPBEX2EEHx1Wnd6ZBEffzJ/wMJqaZTNrAB9cko5pPlEolBA29T143r4fPldcuUDMWFe/PLxorDZ3em+/L6yD08Gh3zaYYPK/FJt9cS4nIQShRwCakAma4WAx9IWQtEomkOqMjE5PCXTSCKuJgtu6iWilIrvfYoxtRnjqMZ7dtRcRhiHAQT2Rw29YnUKk3cPyZZ2Kiyd3t6cIws80XcGDXbnQtX4VaMoFYNCHQonRoPxatOAE1L4bZZgPxmI9kPI2Rn/4SX7v+47jpezfjC1/5smT31VIR2WQU6c4O3H7PYxhLLkLgaMLDr+LYBJJdnSakA2GtKtg1dEwSwhsOQkQd4Ltf/DiqjbpACWvksiARH34ihngyhVQijrjr4RNvWCcQK9vWhoMHhnH8KS9Hun2glYCp16D30cVXmKHJnEAMYVYi8sC40kz4aICEQPx8xfCKa/nQ6UnpIPgwbcLH95eQzzjWbIiX5hcTu3y+ID8T/F+rolotI5vLoZC33gsoFkstz8aNFCG0aDSQTCYEY4uXZvJuYBITYEYU5jeEMPTW1svyPrjk/Dfvk/ekWFmTZ9fT9eC9KFOiCSbtwSdMkIRcI5IaJkkDXxwWPa4a6FySyNfyveiJufn5x8JC+ZmJZIxUNpJyE/F3NJKQVWEkrAlk4cWLowit5Qhi0i/ChInhfdj04J9QKx2WB8qL5A3EEwl8/Y67sHt6Bj2LliK7cBDFZk08ZcKPoloowWvWMT5ZQK2/R3BTMh7H9J7dOPWsc9Hwo2jEkxg5chh9pAL3D+Oa40/BX/76F5x51jlYu3Yt3KCB/fv3YdUJa/HgE09jp98PxzADfFCB4wF8AOTOuNj0ULUK4CptFAT0Sg4ivocbb/go3KbSSpLANDT59KMR+LEo4umUwIWo4+Ctp/biuKWLBcaMjU9gxZqTEUv2InAB31WPQwO1WJafw0inibDmDYQfwrQ0FCJEIp4YsKv7UxZdvZPwJAotJEnT8G4pQBq5sg9zzAJ/j8akhk+zVCxtowtZDn7pJqQ3r8GPaMIsmJsenQZKGEMKsKpshvXafB3pOkIhvo5Q0CZ6rQ1ukvdqTZkiZVf4Psp0xGJMLn3MTE2K99VrdmTzM/HUtWmYqEN8rYl1e3ubrIF1EIww3HyFQsH8vhqxpRyz2Yxet+QJ+mx4rfx8uzn5f/KaOSNv2Ti2bXoIh597QPhywhAJ/9EIIn4U6XgSM1MzmE5m8M277kf/mlUo1Kqy+2hATiOAHzYwumcY4dIlsrMy2RzGd+/EKy+6BFue34Wh41bh4MghdORyaEwVcNXgMrj5Au666y/4zKc/LSHnc5/9LM4/7wI8/czT6L7oXUConmBB0MBEqYpCPAnH9+RPWG+gVmKGrsbjClvgyIO66X8/CadeERigbkE5bYZMN+Ijkogjl0zDibq4cNBBRyaKtq4uyU2OP/E0JDN9spk8kCJUik4igXiqOQ5aeGg/2mJw6HFpGI2GJlZNUnOxmIE5+qCbskmUY+aDsoYuSVOdSZty+jRoMic0GqX+FIcDZsNK6NddJCwKeWzzmnqDSWoEEU83Eg2AtC6TT64VoV46o/CHcCSVSohHnp6eRlsu14qe3KiMJjQawjHif3pQjQJz0MayRb5gZI0c4+PjyOVyqDcC2Th8H16/Ta71PtWRWnjGdWYuYZPN+d/5ejom6zRsDYE5WSymuJ+xhkwSN/OckQuUCVBrVHHPz76IycOH0NGTU2ZCFqchF3p07AhSqTSmi0WEHb341YuHECai8GlUoYN6qYyMH8GmRx9H9ykno1ZvCsadPjqGVCyBSEc3kt39mJieRFc6J2E350dQfnQbpg7uwve//h2EzTru/du9uOK1r8PR6QncvrcOh06YoT5o0gGiRqosogWSmB9DfmZaiiLi2QXT0s5D/Pr730JxYlgwIheYVJ6ETfK29DTJODKZnGDO6y46Hou70+Jxho9MYNExx6Ktd4W8jxehsWlOYB8EcaPgVIce3lfGyNfEshWiQ83wSWHaDTJHPWpxxdJ7EimYyLNgEyon7RqIZBNLTbIMviZul2KQa5JNX5wR3996e1KW3DSJZELWRCKIxfl+xBR0NFmVTcZrbRWZPKX2XEIKfmZNII+sI3MTfq5sRtJ5WiCiFyevL/cMvISR4rVXK1WJbGSICHEZcZRNUWKA70P7YiQL+axNDsT/p2Oi01ToJE8DTUm61Q64+RhVeB0SXcibMwm1ntxinHv/fBtm9mzQB+KGgpvqVb1o7jZ6En4gMXuhOIPnollsnimJFy0WZhFzPITlCp7Z+CQWrFmDRiqFTK4dCd+FFwDlaBxee6fEERr5nhd24YQ1x2N6/CgOP/AgfvH5G5klYveLu7Fu3YkoFKdxx3PjKCCJGm861B1eLpWQTKUQZXjkYhcLiPiK/4yvlV285cG78cSGv7aSPMIq9eQxhC4QiceQSmfF2/3bucdixWCncOileoDOnn5ku4+VzL0ZzoVFegk+aBoTF5SwhQ8nbCoHb3E1F12LOU1hSZSZUQyq9KMDhn2+h7AGBkpIBc9l8lTVPEoMWw2OUMSGbWUUlH4Tlmk2L+vB968bHrs9l20Vg/jsYtGYvJafRWNjUmjDvkITGrneBw1e4Y/doNxUSiXyORBmcZMLnGXy3LpH5bfnIg4T3IZc23wPzgSV/L6lRgWDCwSKGHilntxCwmq9LrkFr9NWOPk8uTnmqFg+E42UZJYkh5hv5Ew9/vTTG9Gceh6VBiuDIZLJlFxgJBIXg58Yn5QdyDcuV/Ko+z5+PVlANJlDpVjE9PikYOQtTzyFVSesw2QihnSmDYM9XZg4fARDx64AU93Ozm4MdPViw3334YR1a3Bo2w6MbX4Gf/nWLahXyvKACXM8P8Ctj2zGeKRPWBKijkqtibBexWOPP4FXnP9K8eBOuQpCdcWqmmmTRuzyGvjCpz5sqn+MSprQsOIZuo7g8lQ6I+Xt15/QhuMGO5HK5RDPtCGRzqGt7zgJgSTzaCSKYU0CZYyWRs6Fjws+VXgwn4MWVqMZyAO17ElZkrVQwj3DPr8iTGaF5gzgR0n51TSBMzDEbmCl1Qg39AHzuZRKNDZ+blMMQXFvFbEocW2+RSGSiyb0UV47RNJwzbyeXDar+Yrvo0iGw8gCfM8XrjoWVzimnpLMRkxYEK44jZfXbtkY3pcWvLRARIPmz3gz/Hy7PtwcvX19qJTLsja2YMcI5LmK+XlNgrsp7SiVkEqllIkivDHRlc+GtkoIyXXjhmpw/RSuCLlp+MYQD9z6dUyO7BGKiGFDsHgsiZ///DeIxtNoooGjM0VcedlFiDoV1Cp1/HG6gmpCNQ4zs7MCCXZvew5LFx2DA3uGkWzrxJKTViIMqugeXIJ6qg1138XRo+NoTOfRs2gBjmzfjsahw/jL125CqZgnokI8GkfokQIDyrVZ1Ko11JsBim4c246Use3AJFKdXeDte/TQzKqFH1ZP47sOujCLr3z2Y2i6xJOhPgipLjrwGP7iMTE+Gth7z10Ir1bAytUnIJ7KoQkfbf3Hi74Eji8P1H7RG1r4QY/IqNGoVw2u1o0ghRUmwVxdU9SREr/Rb9CTCzyhxKFhWZOaKcxoos979sQzkWLTSiNDvHi/kLkSkzm9Kgn3hAz8gZT0AwQNIzWQjcKcgkmghndeh+hPKFswLAd/xvemkSfiCdQbyucrTclyv7I/3OzcXJYB4c+FZaI8gbideYzrSXGL8g6BEyaZpdPkxrBBl5CCEaoVhE2ZnoZucxUbUYi7SaEqlalRk/fN+yBTZelFpXcN7g8ZYzUoIQxd3P3zr2L26B7ZDfzwjo52bH7iOTzwt0eQHRiCl4jiz49sxkBnAh/7tzeCHHu1cwi37TuIQ4eGZRFIW+XHJ9EWS+PQYztQrjRQCCtYdelZOPUV52Oi4aDpepgpzKIwO4Ml/UOIHTiM665+M3ojMRRKEygVp4GAFdcKwloTDTIkTXqnOkpNJoGAk+3G09MJlLw4QM8o+JSFIA3hRAtes4rvfeFjAo/kwRpjCx0XDqmumDJGXMx3nr0ImcY0Vp20Hsl0O/KlKgaWniLaEBq5GGJUIRvvUzlv4syKvEezzjBq9RaOJom+0bywUlutigFaeCLsDDU4hsvmU6DR22sl9adYXL/bQotuCCaxmty6Ljlz0oKe5DhzmJ33S8JOPSHZFQvmCGf4M+Jta8C8F763eFzjIWmsIkPwXBQLRYGI5XJJc4kmIxrzAVKNqh1h5FHoRQEdYVMdHmURvlKLtuLMzcH1YIKsBTI1SGJpSZR9HzXzd4Ff9XrLq9tCF3/Oz+YGsdDIVl4191BI6VRLM6FQV6xGBU387bafYOrAEwTkImBKJjKIxbP48Tduxv7hI1i6/FjMVAP0Lsri7PXHghihnszg5p3DyBfzqn6Dln0rhyZR3H8UJQlFAY5/7VlYfdY5GKvUkcnlcODQEZzXuwBXX3ARUhQklQsoF8ZQmhkXA282tdgh1J/haCUnCByUa1U0/QzKYQIvuEvwwJ23IZtKY3BoETJtnYjEIujp6UKpXMQPP/9RYVxELMXAxfdkmu34cKNxJJIxWdjLT+hEKpjFyuNXo3dgAOV8EYvWnk8EjrqUpl0xSov/hMvFXOEhEF5ZE0NiRhq8KvV81E1CxNczRFveV4yTdQpbjTWAVyt2et/qGdVr2aRVKUoqARUTs9DCpIyUoU1E1eE4gsktBULoIbkES8PG4kWHIgWpQJgXKXaR8TBQQa+D2FyFYvSchAx8FqVisbUmWh33RC1KLp92xShJYxYywOBrGjY9vOYnor6SaKXRSaUHCls0URaIyXWVnETXV4RfhC+Fkty3VnQZtUhjxlqJtOQT00cOipGHrg8vbCKoFrDhD99BucbiBrUFAXp7uhCPp4QpOTo8gsdvvRfLz1iNeHsKbtRFom8IX39qh4iP+FApa02nUth170b4TQ+lQlEYkQWvWIOTL7sUO4ZHsGjhAjjFOn7wT/+K0f370NXbjfHh/Sjnj6JamkbQrKiYyTwIhRgMvyHK1SaSmThqVRaxXJTCGJ5+fhh33HUf2rp74afa0Tc4hBWrVyOWyeF7n/kwfDQkobKbRsKnF0EQiUopnaG3PZjBey89Eel0Fzp7c6jWXfQtP0OKWTXjaWyY5wLTG9LALG1HaDCXdM5pLcSriKqPIiRH2RMRSHmYGB9HNOIJ69De3i6JnHhTUpzUdBAfF4tIk9oTOaqW0vkzGgg9t9WxSFk/qskWXyu41RiTCLDEcGMqFDPJpNWqyHWbjSNCMEIYY4D8XXpkugYr8uIGUxVgIBGCkcwyNPxcJq38DEY5emqrUGS0oYcXea3ZPDaHUgNWTZCNVsJ/0M0ETdRFdqzJt5VWcOtMTU2js7NTC3Bmbfl7hHX07M7onu1iRrwoxUwBNj90O8qTR4yGmnJKqtCogaiiMF3As394FMmeLPpPXoa2ZAqjmU7csvEZuI4Hh5lhxEc2ksDOuzfKgyrk86iHAfqPXYxFF56BbM8A6jEf53QvxPtfeyV2bH4GvZ1tGBsdRbk4hpjfRLmQVyBrviyHXK/xIWtiJXhMmABiTOBXd23EXU/sQGdbG2KpFPoXLcLCZatw+89+hAhqUgWloRMTagnYQxjx4EdjYjiO64sXScTieP/lJyIZVLH8ZRchGktqFDC4V6uWc3plKctQHEUPxGzfeCTxQgI0QymWWaMgzBDvSOciehaVI/C6JKkjrjXww6RLqr40Ai96byZ9tsKo3DQNd05y2qxryVuhjkbW+Yq+lm6dEIqQqNmQzWyxuVQxTZJtGRmFS7rRMumMGDXhFb/TY8/MzghEtLJg/j6N3KodPS+iCSRhnhFPEZIJR16viXcXo3ZVHiDwjddu1oXUrBadrNhNr4fJaFubcvqkcefLlsVudm59NFTNLhMFJe+dsIqtG+5AqTjbChuyIwDk8yWMPPUCRvYO48TLz0EmlcTNm3dhvBEiEY1jcnwcR/eOws1XUanXZTEY0shxO4kojrvyQiS6erFgyWJ8+43XIhONYPTgHhw5tB/dne04MrILtUoeHlTPYDXDEsrkIc6VijWMOggNLVepBXj3J24So01kMoimk8jk2jB6YC+a1RpcE/rkxnk3jocg4gpUkxKzo4tLz/O+y89EV6yE4069GI4srDI2sjdEMKVQyhZCLBdeKBbFAFk5tOIhvrdyJEwOlRmx5W6tCIYC6SwOFoO00lNjVEyMtbGATkcTRy3uNAUjWxotnc4IhGHSzeu1ZXaru1EuWo3efuezZaJpjZwJqoUKtopID2wNj0alRSojlWWJPhY3sEXAvBimrURaBojCX43IobApIrAyEUYrnQp3bEJpM1FJ7I1iU/MNfS2vjbDJ4nDaQ62ikGX++zhPPHhnyA+TbNgI9knSJtwKNj14J5p1dmXE5JeHDxxEpqMd1cPT2P3wNhxz3lqsfNlpuPbGn6FWLmNwaBDZRBo7t74ArwHMFvOCp1gwoIFSFPWK696BYuCgf/FifOeN70FK8GoRW57aAJ+JQmUSzVpFoJJNKMRDUVcjnSMKHSTxkzKvejhJQup1XPPBr6HuJZDIZJHM5aTSx6othUfUrggyNMwCjbphCj00bDFy4Z2jWNyXxdWnLsBJL78UsTg9udHFmNKyJI8tfbfClFgkJkUOeip6VqHdpMztSdFCjZghWZssNM9oyuul6kkNtzFAMlRixBKilSO3AitbqqdhSEQxmnZVASqfzzyC28ry2No80ZCE0aoU+T2TyRhGghFIK4TWELm+GlmIqWnkqkch/s+k0wJvGKn5vlbPot7WFcmANkF44o3ZnKLadc0/ZC2I0aX2DmFxCHvkOYgkl7KEujBE8jqjgdHaqtULqY6eeN5KcPm/lt6kClYi9H13/iKUECt8pmbhvFHuVLIUYwe3ozA5ItoLUnRMIEuTBWz7y0acf+3bUO8bxCe+c7NQcpV8HqWZItoSGQzvPyCGQfzFLyl7R6JIn3E8Fq44Dr0LFuKNp5yNK04+R25iz/NPol6aRmlmDIHIBLRcTNzLm+DiJVJp6fBhAkLDIy9fKRVQq5f1QYfArn1H8clv/FKS5ngmLQkQF3J6ZkbuwWUxxXadeBE0hR30JeFih454ANdBW64NH7rkeKxYfy78mFJgkrSZqhw9qG2xUoaiJqFSlXdsydJqJL2OLevbhMp6RIZdal3YyaMGRSPX9jhGGuWONS8hRrdiJkIAGhWpTVtt5PraZE2xrfLdhEn8srDFJpF209Arz/eSTC553SwsqVYpLvdNHp38O++LsKSzo9MUp5QqbZXSLZ4HowOLhKQ/tWJOKbfcj6ES6alJUzLy2CjGPMzCPysi45rzGdImpc2OG5mb0W4V0sXmc0S3ZCKC0JlctZ3bHg95AbVK0YS/htHfB1gAACAASURBVOgsiCtJ24UNarhrqFUL8pqgVkc0Esem2/6KWszDeP8C/P7u+xBLxqXi5zYdHB4ZhtsM8da3vBU//9nPpIjDCilD3tJXnYmuY5ait6cf6UaAG993PRrNEPt2P4vy9AjCeh6ewwSiKp6NOFXwYxiivaMf9dAVCDJ1dASF/ASaDdVIi0d0AhRmqvhnQpZ4HG1dnZJP0JNMTk0JJhddiwmZxOAi8jKMCRtGbBmbnuo/L1iGdWdfAi8ab8lOBbZJ8qj0HxdfmiLEk2sxxvZPKvVF7t6VriH+2+pX9KEqYyMRwfRzipqP98NoRcdAeo00mckJzHM1lUcVUNHradKpTRgqeqpI0sqNbZNh8fAiltL+TAsnbDOIYFqyOAgxPTUtXtDCJL4nWQyphrLrptHEbD4vkco2YLCDSKS7iYT2udbrovHnLqV3ZRShMxF7UDykEJkdSGywkA3iipKSr52rDqsaUqqjJoJzHSxVyvukQ+DCy/WbnIl5jRj56PCekFmr9hTWtSm3yYpUDU3KOWtVhMSRgUn0RCccYOr5nbjvu9/H9v4BzMDHrp3bVcQk7xEIU/Cef3kPvvylLwqOboZN9Pf34ep//Wf88eknsHbtCfj4WYswtPZqEe44tQa2b7oHvUMLMXZon6j34rEIZqcnRRsSNhz0LFwqfZjxaATjh/fJg+R1Mj+1cgN65rf955cRSeWEpvSj7CBJYnpySgsIgus1AeXGcynwilB1x3xEPbnnU3OdxAcuXYt1LzsPrqv9oEodEkaFEmHUAELBz7LJTNMA/07GwxZwpEWtyhY2peeU361J6Z5eW8ripkhFD8XfZ/gW9sFIdIUWo25dvBYrkiUN3JQGp1LifWtNasi52agfkecrUVAiByNtqWgMW1sIZwtaPbSUqGhnDK8v7JOpMgkcMH2rMzMziDF/MQpF4aFdRzaaVE9NBbbVl2t08VbzYnM/jXKaQLLgRQimzkGLdXyddiFpImnb/ezm4WayG5+QqCPXhsnJSXHMfB9uUEsrOrd87/PhiuWrsHj5CvgR4l2uqxo6F5jkfLVcFJ2xlpy1vzDRbOCv138aOyamcPfMLOpkng1Gpq6bF3/FpZfhn695B5Ys6UexmBf9c9CsosHm1XQS5eFHkBg6H/0L1sL3Ytj65L2iiKN2Jaiz4XlaKnZsDqDAKp7KgvoFeVjcoZ7iNTo5GnmVzcy1Mn5/91P43UNbkMqwmToqRp4nXGFSzW4UY+QSYokzo2rA7FyRBCtsAH4Sn3nbuThuHYtBUYFIlge2zIh4dBY+1J7kYQisMe1g6qzUOahAi9hIPZBW5jQaUE5KTy6VSMMoMBkVrEuYaJJF8UqmQdeWv+k9WXsNamWEFDo1qlJgkxYwQhhRC5bR3d2DYrmM0NOOGjYzV/MF3XSegzrXPAgQjyUlCWUiSeO13TdSI3Bd0QwxAtiqp62Q1hg52AdqS/Chg3x+FqlkyjBMmh/wD700P4tTF/idPDqdmmWjuBZMxOWz7ZQEs8bKtmguMh+GlQoFITmmZyaljY4wkLSiUKU//vbHQlbFKH+sNX3k2vtxzMo16B0YRJ3ertYQloUhk4kdvSd/kX82XP8ZHNq3F9siAZ6amkVIL+8AV732Mnz2M59Eb083SoUJFGYOq4GzXFwsosCmjEYD/akGxifLWHnmu2TRGpUCJseGEfVdTB3dDycoyc5WdZztylbBk0hF2RgRJVZVw8nni/L+ew+N4Maf3IN84CKeSCLTlkM5X2gtor1+el5JuunJ6cFNyTvwKNN18Ym3vBonrluD0IsiFk1pAsSQbQo6opswLVzCS3u+wBfB1YYzZ+LLh2fFT7aYYUc0qM6lJp9vy+d0RYRpklCTmyaUMU0HSptq/sSoKyX+RhXbHrkTs1OzUvxi6B4cGpI1YaO20KUm4VavTsqY2h6lXh1i72RaDNCLELJ5iEbjkiDXeLMm6fR9dQZkcAg/KtSec/25cR0f9PK8d94TGqE0wDCXiKWYHEakc0rqcdIQ7cOXUR/MB6mkZvKq+Yh6fXLypnrKSBGLS7RSYdicvEJyDcoHqlWxoXRGu4FoN2zMECP/4x9uD/Oz02hUZlCvsm2pgsULFmFk+CCicR+xRAK53sVYumwFquUGSmWdn1GrNbHpR7dgxz13wkMEDyVdTER8xD0fs6NHsPfFXSKWyU9PSkGCN0J98qGRAzi49zkJxyz3h6Uizn7NNSJvrZcLGD98EJXSLILaDBpVNiDojRK/ajOt4mFhSITWpJKP5XKGO+24OTA8jC27DuKXdz6JWCKFJAX2putdeHITKhXz8iGpdxNPZuZ7BK6Db33on7Cgt0eM3GHskHYYfRA0NP4ucaJABdNXqS1c2p/I99POHKW8+NDyhbxcu5bFrZTUkcSO18AqI3+u8EfqsvK7hDFMEun1eI18qIy00pjgudjwx5+IjojRQcaH+JTdRqk4n6vQit5GMbeNahoZSGkqO+UEZlIAmOx5EgllUxPOGt2M42kOFPXYS6nRibp+YTgCU5mFJtHsisp1dErC6viEOS4a7DCTqmQdU1OTqNcDdPf2CATj5AheO2W1VN7xeinaFVpTorCOJLGQk59BByzfpYlamRnr+MROtmx5NszPzqJcKaNUKgisKJcLshRBrSTip2iUs0U8HDx0BP/7NY54oDcIsSQaxwXt3TjCUBlN44pv3IBlC5egrS2NicMHMTM7jaR0TodYcdJpmC4UpBF5ZnwUe3fvEPzoeyGGlq5HZ1e/4MTDxONOgFp5CsX8mGGXTVnf4DDeLA2no71DjYb9foampJGV6008+dQz+NvjO7B9eAYZNkX4BiIY1kMMyIRW14kg15YT2EBKrVxlEuPhhv94K5YPdcONZoSl0cZfGrkWMOomsSFDoO8XSAFFk031vjac8/8tnWe7ZWx4JjSx0UWkrMbrcuPwvSw9pwU7V0ZESAVS+GyKzuq4/3c/Ql/fANraVElov1QIZYpSlusX/ZYWouxrtfpIA7fUrNYAGF2sLJfRUwyoqYWrptmASq+aAk1zrsGDHlf4e3MxlnyQWSh2s/nKGnHmj4jXKFk23rql44lkVPsS0aFKMl9FJMIhqkSWpqn56PhR4frJAslG4MQdTibIFyqhhJ4qu4BKgsfYS8hycak4g6BWQ7FAiqeJeo2l9gD5UhG3/ea3+O3Pf4FfvfMaXPuNz+Kzb7sWfeuOxcpzT8K69evxu9/dgb179+LIyDg2vbAbTjSNYwb6cXhiAkMDfXjVRRcKG9K/eAmWrzoVPb39clHkzMdH9gNBGa5TxczUhIxZ4LAcFUZpUYiUHXEmZaT0nDrERznSaDSBHTt34cV9o/jhnx5DKpFmjGt5Az4+60WZ7bNw3NPbg5npGTHy6eIMfMfH+99+OdYt7kGqrZugQaZvMYnu6OhQ+GGSOkZRGiNzGXas8BpswmRL+ZYJ4Hfeh/054RWTPbILTNxsdc82NZN3p3H7TIw9VhDnCbA4NEm01A7GdjwOis6YA9iEzBo3X6NVSWUs2N5o4Yt4PBqckQ3b4ozVlNt6AN+D1ylN2oSlBjrw9+XvZmPyu+XrVXY+t8ksbLKFK3t9Vs8uZACvzo6SsLNnyMaQGTO5nq1PKCOlUckyRGT+amQFGX2svnZ0fFIqnsRMoltmqKxWxcgpgqqVSiiX8lKenRg7jB98/9uaDNYp6HdxZhBBKdbE3tFRHBtrQ+7EJSg4dRw8eAD5QolbHnV40v2OwENFksgG+od6cc6pp2HiyBG84wMfB1JtSGTapPikRk4Z7wya/CzpIWXCOxfGfT8uCQaNq0yMz9BtPMfs1DSOTsxgYvwovnPbo5itNGWQkJbGzT0SKpCpoLjHVbjCRed7lmpl0dpccvoqXHr2WsQzOaRTHaLtilD+a4pJHKsnfLVr5o7M06doNVI1GDJajRGmUm7RdoRXjEbKW6tH5TXIYCA2ObOhIcFuHuOFzZgHFllEBCdJqkIaqQO8uImCY7juSw1Q9D5GyyJsC/MG14rerItVdWYrAsigIUYl9smqWEokvjFdIxq5DkIyTHVLvmAMXHRBc2MtBBcbz203w3zNjI12ttJpx0nMbRwTC0JT+DMOTQtEqmFn1VsSczbkciMyTwgIXxw4W3e8IFcq8/AQoqurC6l4whRXlCrj06Xx/cc1b0G9RqMvm2lNDhY3XCzwgc2Og4FSGe2JOMZidZR5QYbiUuPUMr0MLJK2JB/v+a+PSTfPopUn4OH7HsRV//wvaFY4dKaEI8MvgsWvarmAeqOkCZ0pp3PRct2LJDmamRyTa+OAIXoyGlUhX5QJXXk2cZSq+N7P70NIHQeXg91zpil67qHPSRokMdNWdKw9pg/vOG8V2jsHkMy1IRZTbC8N0y7lo6Z4JBJR5ev5+1KVFY04GxrIYTdkGpnFkvah8ndkvATbDs3EK96blvVVE8IiXQufG3hliyE2SWM2N7Zzo4yrYy7B6xcow/s1lKnAoab2jCo7JE/nJdBGPCypQnOttBvbzib/ZzCyjMKY92Wjoj5vM92K/a2mj3S+TFh8u3EOUhgyjBGvTbC9TZLFc+sULB1zqF3L1hHb39M2pbmvVl8Y6wFGc+787d57Q940s2qrc8hk2jT7Nbzu+MQUvnzDp1CZOIjp2Vk0jCJMOksCF2chgqc9dss1sQYRFKNNHHH4gLRzY+HgQEt5x8yaN0fp6kdu/CWS7R2YnpzAc48/jPNfexmCug5rHBvZg2TMwczUUQQBp0pVVXVKI4CDRctOwsxMHqiXUS5MolaaRd0kgMViWZtsoxHs33cAz+8ZxW/v3ypzVgg7RAogE9jUW7GiZ0VE8t3l7MMQHZEYPvGuc5HOZZGIJ+H5CWkccdmZ77Kwoh6mSrlBPKFqwXTaKO4UM4p6rt6QNWtV7OyIMzPFKpbQ9jHruaQlzoxoq8n4jrn+UkkY7YOlRoSsV2ka+dHnJfEmtNHmCO3lpIeWohRHyLmMOrqJ1QsblmaeR7Zj6ZiDWMGYzRekei1tstbIVR1oPbrCFDMUSfaXKcbME9opRNFrksquqYhbqNIyV3HPFm9o4ciqFc1CvfTfZrPMZSOAZ0fu/fInPwy5cFbfLBXCWFIWSytXESnH3/Cx/xIV4sTUhPKvbH9jQSNo4LRmCiPRBoqZODqqAZYELo56dUw5HErZwOIBTSot3OB3trC99aOfR669CyOHJ/C1z3wUN/3fG9E1uBz1RgWlwiSC0rjAImnXcnQx+Sfd1o9YWz/CRhFjI/tQo5BMRlJYDbZqvGWzjB3F7t178LVfPIpYykeD5TaDHxUqaHHFltq1zUrb/vgen3/r2egbHBSDTiUzcLyEts2RYvPjKJbZXGKYFCZRMpGKzIEmnZYF4hg7fgaLL5ZSrJoEVUVXOtqB6yRj8ESjQ2WelqbtlC0bHUUgZgaHBpVpVMYPmsYKO5jUMCjmGvheMr6BRICpNortGbwr3th4UpuUc+Py91oskJ1CaycfsLvcYHBtmuDlz/XZWlhnG7VFxc9qJJkwmfGiPZz2dSqdVwho79NuIIEdVl8uDIs2Ss9PslXVYoV0XHsWqlw43/jSZ0IusIrcPZVwMhWhgs12dEQiuOW7NwqmzBcKEn45UmKoq1eonij5yUQKhwszyGVS6J4qIhfxcSgooug2sGywX9kaU5zg75frIZILjsHlb/pnPPL4Y/jtb3+D173+SnzwuuuU3QkrKE4Ow3NYRCiZkRQ0dA9Di46jmAPD+3fCCarSkcNCSMPw9+rttDhTKBQxOnIYP7j9ARyYrGry2WrEmBNraYVNsTnDJLEoX/e/7z4fqVxWu9E99rkmEQgs4MNUDQ1CLeSUq3VwHgihCaGUVCjNgwgNNWehitCwZtosI4nmCqrbEBWfmaHC5JbJKGEjHyphDR2SLcnz/SOoYmLfc+K2+Qz1S5sLrAHR47YkCZKPaPue/X/rQOzG53del4V2kvNwMq/ZXCrtJZVrGhvmGXnrnk3uMrfZ1YvTxHWDqganFZn+zmhb18YIQYxtfk9ZLDNzUraJQV9GQ6PiNwHo+v6f+tC/hZFITMrf1PuqR6dKLoKoT6+kA2Fuu/U34lGnp6fEWxFvDsXSMlio0AjxwqG96OvqRm8uC2dmFse4MTTdAON+GZmEJomSwJhueY54nqJKrGsRjl93Im67+2/oO/Y4fOFjH0RHgr1FARqVadRLM0alp80CXKJFS1dgZGQE1XJe8LgUTghjmnMzAAUH1+uYmZnGxMQURo6M42d3bMBY2ex+aaCQxyELwerYTCGvmbrnIZ1MoVau4Po3n4KFCxag3tTJBXxIsVgC1VoTqWw7IjHmL9oeR6GXcM5kQoyeIpXKGL5bu4TooUM3IkUQJuDkvjkFi9/tOAjeC2ekC++rsnNRXjKi0ui0AKZzvpnUhrUZTB14QSTB/Oy5B2yaXVvKG9W2a5V4LmnUopYmk3YTGvWTYWPU2wpGZtmdHLo0Xih3LbIAOzzU4AWBgvMMeC5J1TY9fp6Kz7TeMX+zGX/cQiu2OERPrlIDK81SVafdVMoczb1Ghi+Jkf/XO0J21/C1nssOGWJP/ptlbhfJBD0XMDo6gq1bt0oVixizGgRIk6TMF+Bnsjhh5XI8sWMHMp05xJwAiUoNnWUg71UxHRYxMDCoRl5XT0rmplStS4GhIx3DmhNPxGTDwZLV63HhhReBqLJWmkKtOCkcKg8DIAygsVGNqPMPy6hVi5JQaXhj36LO5eDNT05OiYExCR0fn8JzB6Zw29+eMo7ONjSooUuDgVUC+j4yyRTqlSq+et1rkEkmUTP8utTrmg5yuQ7p4KeRlys1ZPlvR3X5LNhk0uyKrwl+588IO2ic9UYTX/zmd7B794tIp5MyjH7VipU45ZRT0J5NS3f9nPA/lM3CjSWjiEmtGdZCijHRqOQBqM+KkSeSadmgekcvNTI1DDUOS7da49C5iyrptQUXrpvNIcQpStKnvZZi5CZK2KjIHMLCHBNKXvJtPuzg/en7mJrAvKZkC19Ei289uKmAWmjfgjdyYfNRuGn+sZ3dUgoDnP+5/q3hli3PY/XxK2Vsc7nMEcAM2REp91KERONimN/w4Aa5uanpaVl4GdhDgVSziVMjGRx1Q5TaE/jJj3+G4UMH8MsvfwP5F17EQXdGKlrc+Q0zDJ+hulxvoNKooj2ZEFXiGWefju7BQXT2H4Nc/0LUggYaxWmksxnkJybks6mx4OxCGRFRLYmRy8MX6amx3yCQErPO6GPUqePg/mH8+b7H8fD2IzpdaR5XTk8pc0LMCGEn6qOXWo+ZWXzyXeegsy0LptBipPWqVALJIlAjzQRUu9HJ2SpfK5rwgFKJJOqqhQJxlwz8cVzcdMsvUSgqG8N+SOG25ZrZvM3uFkcMvn9gAL29vVizejX6ujslvNt8SDyoGejTYOP32H4wIgsfb9rILCMx5/3sVF71nHN4lgUlbeSgwxBdTRjIBhSoaIxcyRrtw+SG4OtaXlRwi67/fJzMf9vZi9Y4CTvmune0AjvnjS34sEaujIrSkHNfLRbGFKTsZ3Lt7VcLk3/m/W8IJRkxeYOo4coNvHjvMxg6eRXQmZbyLUc38EFveupp8fozhaKoxygeygYhTnaSqEVcNNetwGdu+KxSkM0A/33FW2XMw3QHJZYqVJKEqsKG5CbK1Rp6OtrQnk1i4aJFWHPiOnT09KJvxTopESdTaUxNjsIjI0KS3+xSGRncYGQgJuf8Pl9mgOv8vooYuS24cEEYgcZn89i6fS9+dNu9YmwI6PWpRedm1ulP9IRu1JNpYeViBV973+uAZlkqpnyfSrUuhkd4IYJ8em+Pwz+B8ZkpDA4slA1AGS+5fPuASEmya6hUqeHTX/6uSEplYrDo7NkSpjw5P58elGo6GgKPVWGTAusW3KyEfYmIK6X7VSuPw9CCITSnDiDmNVAvlxDPKSxk00mTsNPACWtE1gOrt59jRsSQZWiSLbZVTZI8N6VLJMqmiWG+MVv2RURcFq60GByJHWJ3/D8xTsusyOaZ88Rz+YNOKRPoZAaMWgsXTD/vkAKptOpRFLq5jI23NhTzs+vfc0lIw04ldW6KKOLYzVEKsO/JbVh2zilo+g5q1FKARpfFczueR7mmb0qcfnypiZjM6wjxybtub1FUXLRStYQvXPwGFOPAwLoV6OzpxrNbt2JyfEImYpUqVXRk0kjEXCxavBj9C4bQ1dOFtoGFGFy2VsNrsyz8ue8SoKphsGiik5s4uozXojJhFZGpWMcq9RQbAqViGaOHDuHhrfvxmz8/DsdpYGlHFL1dbVJIKtUqKNcD5GeqcDhCrRHi09e+FomESogp+q/UzAD4ZEK00pKQeap0rLDJOJaEH4mhGbKjPCHKC4EHkaiZFuvivR/6tNBwemqGftlpVax0ah8kJQ/awCFet8kudEYMOgkdYE8cTBjEDcHpZMlYiN7OHIb6e3DMon70dLabMXOahDLP0T5RNSybn8336hb6We/dMkIanRyYofSrXvSc5269p0lELcuhXloFfTRyPjfamcAjGZz0UrhhP1eeu8H1kg/Mg0cW08smMPUY6TDivRnGZ34y67z/Xa8K6Sk4L4OehPhVZasVpGtA9UgBkWW9SObiiPsxmT8ondqROCYnpjA7Po0FR6pYff7LsW3jRnz+9l+h5DIhcVAv1/COd74FSxwfqfEi3OMGsXjdKhwaHsaObc/KzdaqZWEy2KQQxKI4+eT1GOrvl/L6gpUnCHVGL0yFIn/GncrEmN66o71LvCZxGRs6+F4inqIXlO8qPCJMouaB3pd89f59e3H/fRtxwQkVxLwmIg7ZDRUC8cuKZwXfkrGIUdvSi0ymB/DimC37qDay8KOutLyxhY6RKZ3OylzF6Zk8oomcSJfbOruQzKSou1NjDRq4/C3vNpN2lUmZ/yXeULCxqeC1YrT2tspcFwqAZBbhHPXJ95Yo3NAzgur1ssAj9npmEj4iThM9nZ1YeewyrDimRwzUp6rE8M8CQSjvlZmWZFaY5JI9UW5cGZJ55XtZ9rmk7yU38Xcj8Sxu53ep1MqokbkNIhvO4ujWepgk2bYqzqvIymvnYRet+hqYxAgtLFMTXmB6lq+58syQxlApcVF0cqnII3mmjhNB9cAkJqZnsPz049Hk7EBOkpW+PIbZOM6/+Er85D8/iYGTVyFWDrD6opfjuLPOwZZNT+Hm734dkZCjlhvoLoZI1YBV77wMiVgMO3fsEK0G9RAi8eROFUOj12GhhQ9xrvwsWEvW28eFl18mCjVSd+k0u7QDVMi0NHSCFaUA4slFUzE3aYkecnZmFmG1iNHnfwevUoLLzhbDKpCu1HtT6k8wqqHk+PmRmIdsLoNYMofh4QY6Fp+BStWMh6s7SHT2oW9wscx9UaGV6jBmJo9iYmQvhvftwcOPP4HfbdiG9lzHS65tnmM0rMQctuT/aQFFjVyvjUavXUS2QCSbiMYr2ncWuShBLUtxixp+9g42iOtpZHydo2cvtWfjWLZwEIO9vejuSCAt49+0aGZtTvxxaI6NkQviW1huXDkbu2YtTD5v/9rxeXwGdEYvwddmyGiLCxfu3MxQNxNq7S9YTf78TSUb0OpnFCCKI6DsRN7z2jecHcYiroxkI0ZklZBhjRSPaJWbAZ7f8CyimRiOPXWleE4514VvxHN3pn2MbNqMzpevRrrhYWTrLrziXZdhx+ancXR0XPoBKculbLd4tIr1F7wchdkJuRARHolEVrlSGryUbdkW1ipMqJHSYMnbytyNMMRlV1+FUqWOZCqn8/44oL5eRSPQ0RMM44QtMpGWYb/ehBNnqdfFCxtuRr04I58lQ3aMDNZxlZF46ZeWm3llNKZoIo7O/l6MT03Cz12ExWtPQrZ9UJkAP42wXkG1MIPJiVFMHhlGfmpMDxaolKWx+4GNL+Dhp3fLsCBSq5F4SqhbwhfO/pO+2IgHlymIafwVIzZzhhQmaGVTJmcZ2pTXaNkN9Yo6uEcmWcncc0eauhk92aCgTRva7S9cjNGicANwkyR9HdKT8mtYfswQFi9ego5sStiwCPX2QseZpmd+linyBMKLsc1Q5bACwyjjZRWXzfLsxZRJXqp2ZLIvm4Kctpnga3x8qzLKJ2JtRMbxmW79+SyLjTLca3L/omhUR+Fc/+aLwnRPVhIobTHS4fUM75QsilDIj+DuH/0Ba84+BR3L+hBhb6TvoK2tHw9+++dYun412lctQdxxcf8Pfo3L3vsWOddz27NbhOFgta9ed3DWxa/GIxs2SIHHHqFH7leYETluT6uixIr8mXoEc7qD6c0kXhHtt+/gkte9XjpdVOralIkBjWZFklsWUKQpl8mqtKhx8itQG92E3VvuF16dRsANIJVuuYZ5YbNl6cofkyLTHkJPZpr3DvZj1lmBJSe9EbV6HuWZcRQnD6OYn0WpQGanjHKjLhpvaeSt1jA+M4n7H38ez+4mw8MJXh6GejvwqnNOk8/etXcUR6emMT41rUcyUnBlKoJ00a0NaEK7YlKdS2i1KVaewMTaiqIs/WcTNlM61A1lyB/B/8Iz25MkdPJWXRSV5kAvRnLOpvGaiHk+errbsWTRADpzGbRl4ojxADFedeiJwlQMzEoBjIpR2S7tB5AN2IIn5sCcefCtxbP/XbRSPzSfHdIEVgYOGRxvkYFcw7+fsTo8640XS/JkO81BIxZ2xOgpggY6Gjn88Mab0HXcQhwdPYJTz305Xv7yc/Hjj3waZ1z7JpE8VpsVjNz1KM5806uw+ZknkcvkRBLLpolE36BIb0XgxBHHrnpYjteVrnc5F8aEZXYBzRPIW3tj1Y+DhHjzhFNnnHseOgcXtCp5dTmiRItDWl3V1jmJEk6IbNzHI7//MsrluuBPOQNTkjtV9dEztrBhiwrT6pptCGbuy4m46fY2jE1MoHvV1SjPcuoVD7uiTkX7KaiBrQAAIABJREFUERukP+s11AOV//Jns4VZ3PXgFrx4aEbW96uf+zCGt280Y9HY7c8xbxEk0hm0dQ4Iri8EUYwcOoRHn96CXbt26XMx0IBxSQ4CsHJW02QsntvROS0KddSYjUykpdybf6925o6teGpRiRMQODOd9iDtF8LahHRIMnqOVCPHSegJcZ5D448gl/KRjYZYtGghhkgJp1T2oNMF5kVLwUB6jXbyQEujYrUopgilOYHB9EZ81qIR5b4tl6/WIq8XyOvCue7UNeGF//Y2GQxUlmqWagRmpqaxZ8fz2Pz0M5iamJaxCQxZQ8uXIRKPIhZP4Omf/Q5tPZ046a1XoFmYwdP334+lqU6UE1GM1fM4OjaKoYULsHBwIeK5dmzetEkWxtJI9DSJeFQLGDREc6HWe9uwxe/2pDCryGMHDYcCveHtb2dpQoyUencmpGy8ViqRXLSKkOhjDmy6A2MHtrfUbELjmWNXJKoKrccHOW+h+FBlUKjVWOjm5IPn5zdyZ6Jc1+4a2VhmGBCLXvw3e1J5DeVSDVP5Eu5/9GnsPVzAV/77Ohza9Rz8oCZFKDZhCANiVIwJJrG5LqSz7Uik28DKaYy8vB8VCPjhj/03Ro5OyTlJjG7zcbDMRW/9TNkN1aWop5PZL1QUtiqICnWEobC6HuPirYCKz8pGApscM7lracFF8MYR1aRxzTx2M1udKa50KrlM8gN0ZdNYsngAPd05ZBJRpGMcg8JmFCo8Ca9ohXYrc/PodQnDIn9T7CaV0Fb/qxWDab5i10PymF/8+7Uhvd1IUMPTW7bi6NQU4skELr7kNdLQ0NHZgdDiVsE6Gm46vShu/j8fxWvefy0aHW0yCmB2YgruwQnc+ptf4bhXvQK9/X0idoq6Dva+sB21fBmNUJsAeNPMAXhz9uFquFO6z05MpXFLWDaiMGvk9GCpVBar15+E5WvWaNGnxqm3ZUlC9PWKO/lgB3MN/Pnn30C5UFJo4pOqY4gOZSoAr587QR6gyXL0c3UcgoRVKYZo8kVjbOfJG+ExKDs8kUOZB+YOxJyMbPxZtc4T2yooVmo4MjGFJzY9j/e9++0Y3/ucGUKkbXUy99Ak18w9Mm3tiMbS8iwy2U7kOnpkYFKW804cB8Ojo3j7v/xHS0PT8thiELagYmOgTnid+zIGYdZ2Pra14wJl4tnfleXnb37rRcUpGApUxgyaxgbmF8KqmCNolEvXmeMcL8L1JESW06zDAPGIh3TcRyYTFxr02CWLpHYS1rWhWRxVa8CQOS9Vjs6xVKZiejsY1UYpuYc3nbw6PGHRYnRwVFoqjcRgHyKLF8HNZuRMzIhwwIp59ahvF1HXw70//CkOb96Oa77/VQmjI4dHJLEZyHXh9q98C6/893eAMlF+rTpuBX598w/Ew4pHYebP5EqMXauN1nAUblmds1WkKSakndmBjrwectP0qG9829tQpYyUYxcqZTQpfJKxcqywcpPVse3+H+PwoQOSwIknliRW1WyxKDecOBEtbduKxjxjEZjFziBT0ubiUXu/+0gFTsd60+ZF3TxnxlCXocPgWUd4cfgw/vbo08Kdf+ajH8HI9o2SqBEO8gGKxFlOOrZMiUYm8vJ+PI1EModcZx86+vrR3tUPL+LItNrXvf5qjM6yTjBPlWqbB+yhUPN4cessrPFa49Y+0jn1n2L5udOr5+2Ol/yVQqu/h3fy3uIE5gRUunnnvKvl5WVzmBzA6t6NVk0ku1HOb3eaYleu08BgbxZLFy9Bd0cWybgeZ+66zAFM6x73sjlTR3MsQ8NuuPtWTe+awPTBQ3jxwceQ4vnrg71YeMbL4La1IzTejAZKnjmYKODWT9yA5a94GZae/3Lp7pYgwgE0rodHvvdTnPauN2CmWpbkpVyYxeZHHhHj476Xs+09NahYVI1dMbEZ72uW0hIdFo/RG2i3DR+AdsdTunrKmWeib/EiaTSQGeY0dDPHhOzD0Rfuw55nHkWpStaGcIPJExee/Dm75NWr88GKhzLHlEiGbkQ/8nfpzjHdJjTy7m7sGZlBvf1UHZ0gVGZVMOpssYgt23Zi54ujqBI7A7juX/4J+f3bEeFMd86acfSQKCvztUyI0HueFrvi6SxSmXYksz3oGRhCtr0bqWxSZrH/1//5IB7bvuclhqdrpT/SZgUD+oyO2+JVTdzm/6rZYEJMzPVszn9FK/E1P7QR7//j+oXV0Ejwkigxr1Kp82fEo7W8tH29RkTlyeU1xPGGHpUpaNKNxT+Muk3kMkn0dUSwZuUy9Ob0sF29VlM5feLhu2R0M6tndpxu1HHxzJ/ugz82juxAL/zONjT72xHlyQO1BqLDY7jrB7fg9V/8OOT4Uhlsr4MoaYS777wfjXQMi09bL0zNhr/chbEjY7I0vqcTYVl80iYNPWeeVSxSU1wUncc393CEum6dOkZIUtPQhVDmevD6r3z7m4UP5u9T40FDY2GkMvoMnuTw0oI5a95RcRG9A3e60IIxUom22DJXFLIeT9aHoVeoL5PIer5Ah8NTBZRiJ6JU4UnTFWzfeQjPPLtLxFqyzFKJ83D+6evQn/ZlpqQ9hSIZV8ms0IeG3eDa6EnEqsdJppJIZdqQ7ViArv6FyHR2SoGMwrlPfuLD+OOGzS/hzy1G1tX7xzJWJv0C71gSDzlrhj2kVHIylBFTExETftGTEoIAToMRzjiBf6BPsUyOsFDzNpZcRQvSmKv6u+jCn86HF2L684Yb8VrVaemze8nGI5kt0DRENurjPa8/Q9bPvqc8w81P3BeKWo5Ym4ODSHdR2lksIeICUwdGcPTp7UhwPNtQP9y+HvzhK99CuqcNr/rgvxsFoMIJJhyCQ188iPv/+Becc82bsXjhAvzou99riaXY/CAaDXPQE+fH6AxAHnCqD0bIr9ZBpzYb153JaEF60P6d05xYLV22+jiccOJJ8vlsyqYUNizsxcN/+QUq03mBD9IZY96Xm4yOzvVZfqf4SotNEubmlastI8A9Rx2Inu7Aa46go6cL44Uq7tsexZNbX0C1aqAO2RiT4Qeuj6HOLM5ddxyK+SmJhIR8rPJyLrk2bDDE22m9Kq21JzWwVpFIZdHWsQB9i5Yh1dEmBp6MJ3DDDZ/A7+975v/j9ueSrjnO30ZJvUnFrw7qaPDEOvCI9iZWLhlAd287Nj61DcWqi8BLwmViLN0+9Rast9LXf+TlpR3CGLH14q0I8HeKQfv7klDayuY8VsX+3tz9zLFfrdeb8zuZCx23sAuXnHGcOE2dvqVjoJ0H7/mdeHKZD2KOCRFIQk7U0T5DHpkTj/jYeuc9GHDj+NOdt+PVb34bEuuOlxKtHg7K2Rgc+BMgWqvj9//zbbzm49fhT3+8A41iqTVxiZ5cEk6ZI+jCj+qUJqnSmZkadi1kqq0MbdfwIx5QZnvoNFsaNPn8zrZ21MImrnr72ySS5DkEtDCBZ++9BYePjiFoROE01ZOrkXN6LRMZLUCxOiae3DNH8olUV+mqeU+2dQaoRpsIegd7MZYv44af7ESACByPgi3TYWOKMSuXL8WJCzowdnRKWaRGtdVWyFxA8gNfW9asl9Lh+zrejX9P59oRiXehf9FS5Hp6VKQVi+OGz30cd9y/uaXrmIMic1HQcujzjZyeXD6j6SH0injw9o+jPLMZPjifHAgjKgmOZ9djfCaCq6/5kFRMbbPwPzJy+9nSbjfPk1sDls//OyOfvwnEkI3EQOog8/TocxJeo4FpJaA820BP36CzuvLcEzGY1XkvMriWJ2+wQv/Avb8L2eYm49NME62Ecx7zV9ATwFj5khMkggD3f/0mHDkwjFWnrEPSjaNj1Qo00glEU3ERx9ALF2tFPP/bv6L/5evx0IMPSpgnFNLOFF2BWFRZlQh7KnlRNCg7opfGbRIx2zpFjGr5YJkYazjgeCyKbCojldpzL75QWsiOjB5EdXQj9u/ei0qFI4HpHrT9THlZ8shKNRG3an5AOpFjj3UzCa6jd5VESvUvwq4YTM4HsXT5Uhw8Mob//c1hSZQa9shBVhrDJt7+ustxZHgvygU2fpgRcWaWiXyur22HNHL5kk2sh0rZ2YGEEmSRYul29C1Yiq5+ygaycIIKPvLRj+GBZ3bAc/WQBIVXLw3nL/W2JlKyLuC4+N4NV2Kg4ygaFT0yUKbYptLwY2mZSsD2PhalxqYCXP/53+K5veT3qSbUqMo2wH/09ffY3f5bVI4GX7d+ZoRVekzk3Ki4OVxtc4S5NjkLZZRp08jKaWDvuOAE+FLrcKTBRCliF86mjX8L5ZDPss6Tts3MMi9bjq9T0C1KumoNP33fR3DsOWdg/RWXIokIhp9+Bod37pNz6lefdzYOzfIIxCg64knc/JNbUCyXtJBiEgkRzxjOVabC0gdKaPEQeCo75RxxzY71iDxlBXRalByl19JUcExcBG2ZNHK5LNLZpAyd6c9VsfPZBzB+RI8mCQM9hk+6/eUUNQX50sHjUSDIA1lDma/IhZGDdyVp4zWYTho55Znjq+coxJNOW48nNm/HzXfPahMxN6vj4dKLLkB54hAKM5NSLOGEWjYPWbqNUEk7rthlRANVRkLK4WI3Cl2E75VReAmk2zvQPbAYXQNL0N3bjxdfeBYf//TnsXt0TPT/4vVbCfyc7mW+walxOOhOBfjl967C1KHd8MiPM6KY4wSjiQSiiSxiqTbEEhn4bKIOfanYThZL+OAnfo3NO9nn67TK5v/Q0q0Gfd5/alGKdRhzXrhh/+QajZdv8f3zfs9GOOHy5zVyW5zOl2ZjHl5zykIkYzpYSAzfRErnyYfvDolhbOc2pbZ2IKMNPdR/NxwHRx5+HBt+fjve+KVPomQ+UErefNPZIvZueALxRojMsUM4UJvF4488ak7snRPyiDZFSrxWr6JhWaCB4betDpwXqif96tnplnqyzIncSMRHWy6DBUMDMorulFNPQn7vPdj05CbkC1Wp0skZOnKMChGHFkJEpyxG7CGe4DXoURzi1f25I7NdKV7N0ytLGCW8cXHeZa/GH++8H7c+WkLgxtCWSeGSc8/EwRe2o1rV660bWYEjx1+xAqeyCW7qeIzGyY2lg+rnK1htTsJr4oPNtXUi09WNnqHlWLJsJR6+5/f4769+G1P5RoublmTL0cm55Iv1SMYWeIDnRHH5hcvwT5f1YvzgfqFO5WwgyjhieqRMIpNCLNWJWLJLmjCEN5cJBhohKKYrVUL86wduxnN7qxK9ZcYJPTw9NfEwXCxbcQwmj45hdHwSEYeKRg6AMkUdyUv+cRSYs21tCrFf841/vtGruC7EikVdWN2fMqfJRYXY4NQ3IgJn44a7Qkn6iAtbs/l0piCNXNrCmjy7voRfvP96uh5c8ckPiRiZHDCxNflizjLkkSW86WipjBtv/j7Gjo5pVmz6CSW8WLWaEuaKmQxlJg9JOFbhiUQjrR7KVuK0MicNv6ZARIPhGUFMcGeqdbzzmmvw2O2fwq4dwyjKNF56cgdVOUyVybU5Ntwc/Sf6bWLzCE2eXpotZ9oFxC9pohAsPzdqgYUo2s+Fl16EX/72Afx1WwNnnHYyuiJNcLCRDs/XJIk8vayrESvRWzNacSPTyKgCVEUhjckYgaHaNIdQA2NfadfAILr6l2H5mrW47Wc34XPf+bk0f7Cxer7RWFbIHoFi/++Wr1+LxNTjKM3O6sP3uVkjcgQhhy/JIbCxCDJtfYgmu+QztXtBE/IWA8KurEoBdz1wAB/7wq2gZtN3I/ji/3wKp65chtLMCBq1gp5j5Cfw/P5pfPHL38TEbF4cRqsRQpSNc1hczh+VQGbyL/O5LT7fJKet3EU0OyFSUeDdb7oAnemkzuB0HZTyhdZRjc72Zx4K6b3nhwF+lMKCQJooUpk0vMPj+PknPoc3f+ETSAz1IhFPq7A/dOUNZ0ZHcf/tf0D9yCSu/vD78LXvfAtT+VkdrskZ23U9rkMSSBq9OZpDDJzezUw9siJ9PVNez/ax2hHePzcJpwZI+Zg9qYkEuttzWL5kMZ7cuhmf/MyX8PQfPondu0dRKasn5YwXEjL1RogKoVejhpjPPs0k2tvSiJJW5IgD6e6WA8JlPeSYkyqLOhUUavRgVM0xB/CQi0Sw7rR1+NldOzBa7MJZxw9icmpaey5FNalDMptUP7YKNIrx2VIotJ2ncIVuUOb+SUe8lq45/Um8rKmuOm4UHZ2dGFyyHMevPxU/uvFL+NYv7zHFNdP3N0+tx8ojXM2REtEMHrrj37DrkT+jYvIsXpPO1vERift6MnV7DslMFolMP+Kpdp1eIId9zUlsRdvi6AYeGz2ILc+GWPfKq1EceV7OXBUlp3gr1RiJ05KGkTb4qTZ4kRQ+94Uv49GNGzGd1+N2tGHEQ3d3Oy545Svw61tvg5w+Y/KuuZY20/xhRE78+SWXXIxr3nEVZkZ3CQHCI7tVhBjAk8NqAeepR+8OybuyoYAXRK/DzF0ekBkfzMrbHV/6Jl7ctAkf+O2PRe3nV+vY+uCj2LLhIezftw+ztQoWn7AKp5//CrT39uK2X/wK49NTAlcaDaX9RHQlwy3N2e2mY4dJGrvj23IJKY5QOisVSdtRLgmpJAct0RHnpxTLVex4YScGB/qxavmxeHbHNrz3P96HvY//AC/sPIRKFdJkzAO6CjUSYQ6WDHUikXSkiUA2F43b4mWdxNOSifIT7ZgINnY3Ak/gwd6DY1gw2I61qxbgtw+M4p3v/iAe/vPtmMoXTc3ATCXgqDgZ9KMnNBOREn/Ti3Ktk7xPYZaUPSKUsc7GdswwiMnICtcTznzZ8eskum148H78+M6HWke66Dmc+nBlsq4HJBwPb7r0FPzrG4/Brqefkj5O60VFHMchmlFPjDyRTiHVlkMik0My149oPGeiLDlqnlA3d4guoQd/f99zz+PFPRNYsuICLe2rIN8kwHMSajaixxOd8JNZeNGEwAi2MYool3+Xw3TjUpke27cVt915H276yR/EkdmpWfq+qhviGvEIzR/88IfoaEugXp5BIFMbdKqtdDYy2nMMH3uQn930oBynYs9gaW9rQzFfkMGf3V3dEj3GDx/Bd655HxYtGED7ooV49rHHcKScR6anExdceTlWrz8R7T29cvhrKDca4KYvfAX7Dw2L163WGmLksnGoS5Hh8qHML+/vSCNGHEfcJw/fhG5TsVIqT/Gq4DLDAklLlfP/6HoPMDnLsgv4zOzM7GzfbHbTQwolEEINEOmC8imgNINGitKkCiJR6QKKFEGRIiAoRaRIlfJRpEiTEkpICOl9N9t3p+z0svNf59zPM8n3X/+/Xl4Jm92Zed/3ee7nvs997nOCGE6ksPTLZTji0EOxfv06zD/xGMTXv4o1a3oRHzGp6Uw+j1nbT0U0SvYhp3lqFLW14NRAMoqxb55Ym9hX9d5DkicRECgWMJCuoHtLEvPmzcBLi/I4eP9DsGndCmSypkOiiSeXpmXoo+l8K810izWG+XNG+adjYhpnxGHk26pk+UZR0FCuY+b/EC8+9zQ29w3j+Xc+0X1hXdJQX2+FuiCgIr572M6Yf9h4DG1Yh2J5BKMFDjmXRFFmj8LDlKFIDeqb6lHbUI/G1mY0tIxFXeMERBqadYoapmiLy7Ma2bxiOrf686Xo7i1g8qx5aipx4aoK0ILcShqzRd6GmvpGhGsbbCyQQqvslQjV4SYGBjpXI54YQG9fDGdddL1ou6I3u9PNL/LpM6bjr/ffr/tVysUwWkyjmCVoYkpoTCfVFZeZQ9GaQSr8iG5wqsb5r9MQqZDJofvjxXjzpZfRvWYVou1tmDlnJ+y+795onzFDxK0xnIKh9Z4YeM61uAI89fdHsHLFSqTzWc1FUm9F+oCFAnaYPgltLQ2oYxRxO3PbLpWvtH1jwQ+qekMrLXbHS+bm6RkcQlNdIwaHE7juppvw7lO/xLKl3YjHMpg0uQOUa6kVisIC045pbjIvtuO7P/9v8M1LInDdsKPGG0fUKZMpY9yEqRiMD+I/S0s4aN99sbFzg6BKGz1jJKeR7qjUBfyG4cJiMGGU5meoi9giJ9zFxSl3NbWi7c/qonWoxLiJ4zVgvWrVamzsH8LargEEOAjBlVhI4bgjD8Q396hDrn8tcllqthQkdOQ7jmqMWJ9cf4aipsYQrQujsa1FIkr1Le2oaxqPcLhOqYpG8Rykyj6IEsayOTp//PobCER3QNvkXXSNypUrW4vUrXVCADW1daita0O4rk1IXCjETWdNG96LdHIAvZtWKE1etnIdfvXbe2zIuSo3Tf3MMG6+6SZ8bd5cVMoFWWFWirSQEafEgmCFPQd2lZmJFFRLBpZ9/q4WOYV0TPPZVJrGto/F1Zdeid0njMdOe+2OfQ7cF509fchxjnK0jGi4TrzqSCiiKRzmdLK7dtDjC08+hVUrVmA4mUS6UJQNR8fYDuw4pQ3hiB3VnNwgl0RFV9VdYJsjz8MN/1/dMCIkpNPmC/K+WfT5EkyaPAU33noLXvnrhYjHUmhuaTDLEqUJzBGdAqqMYG2oQMefRyBYFwihMDyX3+bNsi/T2uZCZmp38EGH4OkX3sEBx16IT997Hxt7elAqmH0JN0KOygEwhwn/sG0RWBNKKlgO05VVi0tXDHkhMuBGt7YpKk8963T869EnsbG3G1uGk8iVR7HX9g0484RdsHH1SoRHKUJE3gddPRgHrGhWCqZ8z0NwjpMTMmChrqEWdc2NaBnbJplqLnIqDTBFoWCRqW8ZBVZD0zyN8wW8+Pjj2P2Ak4GaJhZWFsH9uLwfJdRBIBI+onXNiDR0IEzacKQe4RCxbLv2TWsXo5hLCij4aNFyXH/7g/9nyJmB4MmnnsSUSe3Ip2mDmddMgIRqXV3HZ8pgRKYo2aPpZAzJ4WEEln/xvtIVHhvyd3cXxEqbR9LgIDFRa8Wb429FVbgx6GqQSCT1c3xoLFI5TRQYHcVniz7CG6++iq7uXlEpZ8/aQZGLI1Bqwjh80ttQW7gzxEtFnwoIm1ZX1JHHqDOg0pSQCd1QyCedymBzdy9K5SCuve5ydH/5gIkgSTLDmkAiEaoQtIJ6W0iKx5s1nf7vwrLFaTuNCA1/hwMXqVQeu+0+G0++8gX+55iz8fYbb5pEB2m1HJSgZJ08R+skm8dTMeqaWxJucimYCiuHLjDvzebyoD4ihZNoqyjtdM1Sh3DMccfhy8WfYtWalRJoOviAadhluxBGtmwWxdh3gD3MaiCFHd3+njrKkoMFGdUpQhqRcH1dayNaOsaioW0iahtaJHNn2u0O3xeHpWRDyIEA+ru68eHrb2HOIWdbse6ek0d2tkKBW/9WUxNFbX0rwk0dqG/ke/C0CCE53Ifh3vUKlpT8e/a1j/DQP56tNrYqNcCuu87GIw8/hHJuBOUsNwMFYLeedt4EgPJ9nEorF7KID/dhsH/AFrkWsHIYkyzgzeCQBLVLiIsyyVfu51RuedfMkcLYfq2trboS08mroGaUUhRp3PfHP2HchAmIgoJFNjzAyGD8aWvR2lSQo3l6Uo5DYLQ4vXuYhl3dLKIKV5OJoA1JIp5E7+CwSFk//8U5CMX+YyZMRDpIA3AquqIesJmjDc0/nfUHUxGn8afhDZdCGdJiG1uqADoVSxhJ5dDSMh7PvbEOs/aYh03rNyGZyWroYuL48dZtq/JgyOlhQ8da1bb4rPPrDWsDZfceTqORqUuhaD7xazZs0GD0gu99D8++8BxisR788foFWPHB2zKPGuV0uYcp3Xr6v5jy1gFjj5kHIjYQzUDD/1EFgcjKmPEdaBjbgbrGsYqyXgSWQUfi+FKaryAUDOGDN/6D/r5RzNzvuxqEMCTFY9//F9KsDpOT/xWMoLZuLKJNY9VwqqurRfeG5aaBT138fA4/Ovdy5Ecjii92ggCffvIBykWaQliBKTjapWLbkrl4taViBulkHLHBHkG6ga8+e7tilEx74LQm5BFL9yxDvni00hqbVnPmV0N8nEc2Hxp5FPwg/IDWmbTcmw2c2OAQ6qJhbFz6BeKxAaTSSddW38biw7EYjatgT8lPpRu70Xwx/ZFvF1SD8mhekTOTzmFoOIb+ZALHf+8EHLb/vlj/+V+QSWY0n2iWhER3jLut/FqDFIa5+2l3nzd7Nh0njywq2iS6J4YVsgX0xUrY1FXAUKEJe3/tIOw6Z1ekYgmlcrxHnPOslCgGZDOmkopw0+RuzN1OGKm7msSGNoC1l+1EdZqR8gDaeTZ61m7GB18tw19vOxmLX3vRWY0bRcFvHjuh/L1y4ppV2bhtRsREZ7D6hCmMusZtY9AyaRwaOZzR3IbaSK1ZMnpxFj0YUl5L6B8YwvsvvIyJeyyQehh/jlGfr8YROKqKVS1U1O7mQt2qNBCooSpbI1rHT0N2JI5UKoEMZ2PTGcTiQzj/ijsUDNno2W3XXXD95RciUmtNwVAN01yDlUUDUSPTNGFUmhRyyGVG1IhKJ+ICPgJffvKWIjkLAC5YSh1zB3NR+YXMv/vmCBccZY39sajd53T++HfN8qkjSI+XEN55/l+IDfQ5rRCtLBfJ/G63SGsphWvUlM2dmF+SmNCAtWeq8UKK1NcEOaB0s+jqj+Nbhx+ISjGDaDiPptAmpEcSzmLcpSa+gKky5Dx6YtJn6sS6NMZyS/sSh10yF6MoFioYjuWwuS+HbLkBp190jdKlZJIQltk/eqIaE1fxddymZ7HG+U/qhEsagmhTmQ03aox7D1ArXFXwanKfGH0e3znuBNx0y62YNaMeB+1Sg5Ehs7thu92L/fiF7jeMTxt41Psoa3wdc2ewRc50kJB2RUKkrZM6MGbCZNQ3tyEcrTdXbhrgOp1D5rocZPjo3fexdvlGvPRpCY1NTQqM+fQgotE67DhzO8ycMQ0dk8dx5Lyq57P1GdqEPslsE6bNQl/vFqRTSaSSMQzFkrj2pnsRrG3CH/5wEya2t5sqQJnyeFSlZ8AzrrvqDM0KZVEtAAAgAElEQVRxGiRL4p2d2HnEhwaRiA1LfUw10cov3qswUhtf25waZDcoGxBGbdOn5sL2LX/KP5h/jdlFq01eKqOFxCEKvmczqtoZrd544RkUsrSfNh0PLR43ha+oRQdjFXxGT2Uw83RW25kFRRXewEi0Fu1tbZg8eQoWr1yDO+9/XF00Yq2/+eVF2HuXGezFId7zLga719GByG0qbiwn7mPlujUa3AS8ik2vVOXugwoalz7wmpiLJ0fy6BsqoKu3hJ33mIdDv3syCpkUUumUCndSjcX5YWPHDsEq9EnM1/oQZuvNf2FXmZueejE6bbJcuOYIUWaRx5NgFKiLhPH4M6/g9msPxdpPliAju0hChdbX0CizI+BTYdfkn62AJi9ci1xENIuopDvb3zmrSg4KU5AatE8ch9aJE9HSPg61DXZC+6ktXU6wglh/P9544XX0JWvwz/8MVgOWXztZaqyPltAUrcH20yZir913wezZ22NcexsiUQ40MK0JoX3iDKSzJeQzSQwO9Ei1bOqM7RGONiKdTOp0i9RGxRZlY4mU50gwJIv5dDqBaJTTVGaiZQxtk7lIxuNIxGIokG6dKViGsWrJf7XI+SEVHZz7AW+6ZNhYlIashU+ExFtjSLWKJqM1QDRSi0qRWDv0wMnFEK6KED758AMM9na7QpKbwQv3UD+wiCI1vsNBTJ82Ba1jxhoTLmpy0T5N0UAwxeipshuuVSoVDEXwk1/diIHhQUncsUX28vNPSJmqQCkHN1BbzGZx6a8uQmN9EL+88DQkhjYhEesCygX9TE3QhhMMAzY5NmIw8vSsCaFYNKgxlR1BLF7Chi15bBkJYJ+Dj8eBB3xNmDTvi6gPOdMON1Vo77dp2oJWQNuiZO2jNEzDC7bplYdzqt+lNYzwPCV23W13/P2ee9DTvxrnnTgbPRv6nTD+Vhk1Ugf8F+cnPZ4tBM4zKQmdhk26gt1lyXEIETGKAv97zJhWjJ0yAWMmTEBjKzuetdaR1Zepf73+wusY7hnC60tT2DRsNuYeNRJu4FJcno0MfOyJZFMjaGgI4sC5u+LA/fbCjnN2x8TtZiE2MCgTYZqS9XT3mYComkPqWGi8keuICmXk0Mv5jdY1OS5eukuTC5/TRuB153JpDA30I5fNWX6fzQmACKz58oMKo4B5H1IEJi8UgwuJ3+eiNgYg+eYFHRn8MI21zG957BaE/SbjCWltcMOEOFnCaEQilrS6g8rbqJD6j+f+F6+8/F8Uc3EsvORnuP62e/HdIw7CmScdr89AfUE2Y/i7cmzQgzd2YpYSEzlTx6qrjeC8q/+E/ngMrS1jlWY9+rd7MLGDiloBFHjDKiX885//wr9efRUnHn8sjj/yGyhLS7uM4086D/vP3ROX/fxsSUDzgav3X86jWE5iJDaITCKG7p5O9PX3KV0ZiqXw+doYcjXtGN82DlcuPBuZ2JA8SbkRqNjLIs5SEfPsIaRYR1MuWonzhJRWoxliyTBL3GfTd/SNLq6TfKkoigAtxB95+BGceexMpIY2IZsqoCi5OcvFVRQ7oygtdQ4CODkGi76+KCSq5VIXktEcnOn59FysrEMmbDcJYyaMR9O4DjQ1tjgukcF8yz/7HEs/WY7c6Cge/U/WmGz/P182VOx0IHnCUeg1W0Q+l8Y777+DWE83Whrq0dXViZ6eXgVUpkb8kLJeHzUdeDFjaWleXy9Yk5uOhsHhWrpCFwQu5LJx1AYLiCeGkIonZCxGKDuXyeDzzz5HYNOqT2VxyLSgtbVFO5qrn1/qzgWDSI5QUnhUTsmcjmFhVd9AxdaAikk+QLH5olGTNpCOtQniy1HZGVHxoT7z4ht44l+vIDeSxC9+fgFuveMeHHvkt3Dmqcfq2GEdQPtw1QUV1yV1pkzBcFQXGKEzcLQRGzb3YuHV14o7w2jSMbYVD9/75/8DD5527gWIJeK449Y/YEp7qxZ/rlzGSWdcgJ9fcBb22XMX5Y68bn5mbiy+FqNBLBbD+o1d+PMDDyMeT0ioX8zCEj0589h/7u5Y8N3/QSmXdgYBHKawekZeP5rfNOH8RDJp9zREMpxztHA0ChZ39FJis0VT7JVRpFNpdPf2onvjWny0aBEWnjQHvb39sjgcpZ6868huzcVNtoM5qkcbhFq5ha0T2PUkWKuJpag+AT+TlYmMjOPGd6BtQjsax7fLtp2OzhQU6tzYhQ/f/ADZkQISoy14cRFV0P4/mISOaag01nVu/UAxWaInn3ISvvvtb2Kguwe9XZsxkoiD012EniUrQgoB0z03Nug57kxnGxqbVeCSMWmGAzYvTG5RuZhC75YNGOpZL1cOpn6U8HvzzTcR2Lz6s4pG16qSD1YUqSFRKakoiJKSSevnuqjxzrMZKwZrgujs3ITJkyfrA3KzGBzpCT1upAvU4TZ7v9fe/ggPPfEvLfLfXnMZrrn+ViyYfyROns9FbuNlHNZgrkXMmPAkH15jy1jRBnijiKqotRxuwHE/PEkQ4llnnYWHHnwAb7z8vCwafdF6wg9P1SzjYw8/jAYO5nA8brSM7596Du645Xdoa6mVozSjCFMiRjMueKZdjML5YgULr7pGgv7nnHUGRlJJbOnpx7JlyzE4PIzmxibU1JRw0jHHYPp2kxEJ0BOHC4aLHWrvaySQVitNTfpv5prkk2vKSRGfeiUUI8rJMHigrxe5dBbDiSRWf7UaU6fVYvftapDN8PhNyQCB86s1o9Yp5UC2kCIFFMvFpV/CjUDpPx3zjvchEMHovrVigJLSamuK9OfWMU3omDQeYydPQH0jyVoN6Ovsw8fvfIR0qqL78Z+lwxjINQoGdplM9Q8NL25LSNPwiQXM//nGN/Hdo47A8JZObN60yWjG7LiS5ktDYUpjFwwFo+UmVXw13xCNyq9J/B3SF7jQXSotCe9yGbWROiSSMeHoa1cuQX/XOkmDvPPOOwisXvp+RYMKFLiXGW0BgQJ1+ehVk7VoTIcxcjBUwFiksKkMq5QZAQ27cvOaouEW9O++idTUxEImgOdefQd/e/Rp5JIJ3HL91bjk2t/hgtO+j0O+to92KSGhOppEEYVgoUIYhRAUtcPdWJRHMOj0/MvLrsLqDV1Y+Itf4Jabb8Dhhx2KX154gW46c9X5p5winfFn/vGwk/UNyqtnwenn4fEH7pZ+osnUuaED4vajoxqG5k0aGhrG5dfdJMbc76+/DsXkCAYScYzkcnjw0Scxc/p0pXaMHqUSq5AivnHwPOy/x26IhEbFxykXK0hnuMmDqIvWVt+PqZnVPBX09/epeVUuc3glj0JpBCef+h1Ea9OWlrBg1f+ZLtrzSMcoSZdCNpkS30gggU+JWPpoJNHorNzcdOlg/6BUpu13PaK1TFGCytVFOQ4ATS11GDelHa2Tx6JtzDhsXr0Ra9d0Ip0uI5lhDVaPZz4ZxmiZ3lJukfuWvshtDrVyc6p8Zkd885s45Yc/QPfG1Vi3YpmUBpQic0Cjlhqc5tjhIUEOn0Rq2SiqRX1dk6zPqaJcofASDXdD3Lhhx8+3BqGpLUDuIPR1LRVyWPbZe3j1xecQWL3kLbm/jWY5rV1EuNaEJMUzKVrOx+LBW9CxqcEbpfE4MhedWKa5dpmGNvMoRkY+LEMazOeysbEJ7yxagjvu+zsKqRH88cZrcdFV1+Lqn/8Uc/eYo8FiFhDRxjFaoGKQgXmfEaoshXKafZIRDmJzVy8WXnaFCrbjjzse/3j073j+8cet8A0EcOKppyKbyePlp55AoUwIr4RMPodTf3IhHv3bn0XWkl+Pe23Ln03li7lzPJbAldffoqi98MLzsd24duPhlEu44trfSfR0wYIFeOaZZ1DI5dAyZoyYj8atK+PIww/G3jvvhPoQIciCpof8Zi3mqfhVQMBpqtNNj8ZjwZoyTjnzIBO8L5kAv0GvViBSZoMPlJuVKUeFXJl83vL9fAGpJKWuDT4rZPLIy3qmWCXJFUfZUQ4gwe+XoNogGh1FfaQGjS11GDu+Re4W7737KZLJIrJZnkS0lhxFarQRby2J6fe94n4VrlSq5WDKUAjzjzsWxx97DAY6N2LDyqWysuRpTXKWOPW0inRpLhe0Nhprw2AQdVJhoFteCyJRYuO1qKN0NwIyY1OmoeEXP4Ngolck7andT3MGdpFjfQhsXPzviorEyqiOMEtFuDMsovGLi4D+lF48Xdi1CFd5s8qm5babFOJulDwvbbTr602oXlCcGd+u3NSPW++6H4V0ArffegMu+OXVuPPWm7DzDjPN2luzlFYtG9xoeDPvnhVZZtDkKaXMzU486UeIJxP411PP4sQfzMevL78cc/faE4VyBWece4647P+4/x5NsPA1aMp18unn4u9/vctEfhhNyZsul3V0GiHMmkapTBp33fsQln61HKf/6FTsutN2BlvV1OCpZ1/Aex9+gksWLsQ999yDRDqDBSeeIDZkf/+glHZp5Ugpt/DoKHbeYTq+tudsjG9tQDTMBlrO+BnUa8mlkUyk0NnVjZ+cfxzaxxufp5A1tz2mJ16ov1Q2Kxb/RSKYcZRsQIV/pw4jA4tOYYqu5gpCGxiAypTsyBflkl0sBdHXn0AimcP48U2Yt/8uyJUL2LyuB6kUZe4qcrVjoKEY07srM+hJmMKApwZLwzwYQH00goMP2B9HH3UUUMlj/erVyLJrnorrs/FSRUhzhrlUIlB+TeJabVSbjYue0icMiJE6YvX15ptEtKWRJmMV1NUz6jMlZPHpbGDcXHANuVR5ZiA2t0DYO7D201cqzEO5UPkNVrnM7XgzeIz5ljujmm8gMJKzQLIGDqWALWp7Vh/vv1/o3G1ECZg7ERZcvXEAv7nlDuSzaTzxyMNYcNoZeOzhB9BUz1zYyf06nRNP1vcwFd/X85XVjHI0hBt+fxs+W/wFrrzsUi3YG35/Ex5/8CGsXr8eN9/yB0ybNh3XXfkLcy4LAOlMHmecfT6eevQBVeLehUxdUdlyh7SpuVHThQzWrO3Cn+68E+0dE3D5xWcjo9QjjNFgGBf94nL86Ec/wlNPPYW6aBTnnXE64uzgZXMYisWwbu16Se+lR+gNVFGkZspCAdIjD94Xu2w/BchnkMmkEY+NoLO/H3fcdQHCtSFFvlIpIyqCpq4c1MhIXnVMc3RYX/x7K0R1nzXiZzUWH7hszgtF8UOISlSyZXUES5USwpF6tHe0YOVXq5DOlMBbneXAiDqvZv1CKsvDb/SiEiIZL4Dpkyfh5xeej3I+jUwyLhGp4YFevW+IsDLlQ7iOIlykhuxwzdRG6OIHFZw0DmOAjNY36J4zitfWNUj7MVLXoI4qO6isBzlcrY67716709ejTH6w2QRKDYhUJ/2jVx+pjGkdg6JrQ6taL4+qk7V69Ur541Stqj2nm1GDhY9rDTPSW/Q35zU/g8kNwzfjvysoV0YxmKrgmhv+iGwug6eeeBwnLvghnv3nY6hxUznK811Vrg9vvygYUXOQwkNzrltnRK5sATjjrLPkpnbfPffiuAU/wDN//wde/fdr+McTT+K444/DUd842Lw5g/QPyuDsC36GRx+4x3VuHQ2YprGaYqFtSUWRsEgia009Lrr4EsTjSdx3x026RqUO4Xqc97OFgg25ITilcsDcvXUvUyMjEhzK5UoYjMcxOJRA5+bNWLV2rYYfrMYJqaPX0NiAfCGDkWRWKMOSt25BKESYsYwRDkMTFMjxHtvQgzU+rBssxqT3y3EnpqEq1lEujZq0s+gJfJ1iSTmxmlBFLuashJZWr1iDVIrIVgmpDGSXw7diocy6iK6Au809DM2TZmPL2hUYScaFrHnddrJw+TnCIVPwMuq/zWmSaWpD4dbFZmteLEx6I42O6v7R/Ff0YxaW4ajc9BjJo/X1qsdUPGujmQugwBE3muitZ1SvyMWCn90KfiJZgS8/eLGycvkyzJw+Q29CrFptds7n8YhUty9dnf8kA1FFXZ5uwcTUg9WpIjs+imIp8lTIZdNVG8Bx4ybqQw6mCjjr3J+qW/rUE//E9364AC8++QQKpaxkBRwRcatr8DYDr7bovXyDsw9RmkQ9xNOR4Ws++gje++Aj/Oupp7H9zjvhvY8W4YG7bkek1mgDzJUTqSwuXPhz/PXue5Q5Ux1AN6hiXqGRcK2uw/+fi33hldcKBnzkvj9bGqCUrYR3P/gEr7zxlu7B7bfcqLyYC7hYzKlLSwt0/vxIJotPFn+Jjz7+FAfu/zX09PQgHo9rkbEAE18ok0JDtA4/Pf0InH3ygRBkGiwjPjxsBgPFvAaCGR01rqdrr1FzyNuJ+4hu+jROz9AZXvHU5UnFHmmQM6gA0sND+GLRUmSyZeSKwEia+o3m01pACLvucwjm7nMQli5ZieH+LcbEzOec8oGzKHSbTHWQgpQFI3GF+MWGkxuqtlzahjZYdDJqk+JdEw6jsanZFA/C9WhmM4oiSs1E10pSSivS5p4pjReeApRe6oRnb0H8KaNpeMBE2cVXn75ZYceot3OzdvzUqVORGolVbQMZ/Zi2+AfO6KxjoVgymzqNs9ki8RCibwfny0DHuAnqHxLa4o6MJ9I47Sc/UTR+9smn8b0FC/DsY48iEDTDWYtC9gA9DGiojhMvd97t2mjcqZKpKOOt9z/EPffeh4fuu1fFFzfg9b+/EZ09vXj4L3fbKF2AjdGCpvaff+V/MYvikeM6dExqkMJNpdP5wXgdQRV07DwuvOIaLfI/33qj4CueKvKirIni0ssuE032xuuuFvWAr0UEZHiY8hwUHCJUWMHf/v4PbNrchdN+fCrS6QyGY0l5NHVv6VEakxhJo67edBM/+N870Vg34jxVR5FLJeWLlM2lpfe+LXbnh0qMM+4c3IxZZv6fzqnay+IRmm2M1qN3wyasXL4cI/EiMtkKMrkyMgVjQFYCIfz0shvw4bsfor+nG4UCU0Xn86luLrk6ngvjjKu0nreaWPmClM58dpTbQAUXIdeVLWrCtxHNI9Q3NmkMj02fppYxaGppAWpqq/opzNWVabi0xw+Ha9LMcZtMh8W51Ln6JLBh5UcVeTcSSkMA3Z2dGNNSj+bGBhVCPBr9MSMtaILwQXMD5u5MJGLKrZgLMnIxb6pjp4zQo9PIZuGnwrSmBqlsAaedfbaw9Ccf/yfmnzgfTz/2D5Qq5H4zlw/JF9QTwLzNh+YMCXUSJmJu6UYdfAHGI+vHZ5+HKRMn4bqrrtIGPOdnF6pW+PMtN2ig2DTFLUqxBrE0jLBaBoODg7rZLHhamltde573xZyDn335Nbz677dw2803oiZAe0YbkOjsH8R9f/krWhtq8auLL7K2Obu+tTbtX6YwP8fhSgXccMufMH78BHx//gkYicVRKJFFmca7H3yI/qFhFYKyVsxkUBkt4IN/34LGKIvtAEKVUYyMDCGbTaBSKmC0ZEPaSp2CRvBShzoYdnwgAwAUSL32IPe5Gy9MDcXx1SeLEYvlkEyzBmMaWESWsmuVEH58xkIsWfKF1gDvJV+bs7r+ufj7rkXL6F1FvawgrtrYuKEPG4whqcpOYj4LrheC6Go4uaje1NKGYLhWtIIov8cmUZhEsYhzgeYGsZzbWK/bmHPpvSzgMgBZKlWDwNpl/61YEcNlA4wkGTGyWLViOebM2smNEhm32QxdCQfySGNHkxgr4ZwwWto75DMvW3GXExHeYnQn1GdF6igS6RzOOPdclv94/B+P4vj538PjDz+gYVoIsSHBqVbHEI9hOZhtQxflBdhdtNfzN5gXffGlV6KzqxOPPfCg3vdcLboK/nr7rYIkmUYwwppfjj0wL2ykhkItzXppH2iRxsbteMNKGIqP4JY77sXPLzgfUyaORZ7VPGpw85/ukK35L39+IQKFnHNeDiu35iaiWYGOztEKFl7+axx19NHYY85syUDnizkFi1f+/aYaTDy2991nrtKYgUG6UQ/h1WdvRjQ0Ih4QiZnx2CBKuRGNEbJDari5pSH+wYsazPlGd8Ly/fnv3KxMY1obGvH2q68jPpRGKlNBMl1EhhAhx/fKo5i2wxxMmTYLmzdvRrlkJzXb5JyH5Xtt2+zZdrH5YMjvsZ/CgKTF7aQmagkZOvFOpS0hqhI3CoZld5XFZ7SuCWM6OjTwTDNgnppMc8Vtd4iKUiG3JvicqzWjYF8aFAdNUmXU2LCBdV99VNFUifS+66QZQlI6C6dsfBi5fAotTY32Jk6DcGx7B9IpGrhG0NDSblxhx7DjgqiK4DstQ94kbhL+TDZfwo/OOgt1tSH85a67lSN3d23GcGwAE8eNV1HGytwIXkbx5e9XF6brP7BPaP9GaNJee3PXFlxx9bX44623Coe96JJL8KNTTsHXD9xXpENuTMJLjMDDw2xLA80tZg/O9/BDIYwwvJFcbH7ihq383/3hz9ht19mYf+y3tLEZfS675reidN560/UIlItWFMsivCRzWkJifCD82at+eyMuu/SXaGtpQiqZUmDhZ3nqxZeweXM3mpsacOS3jkAxV0A6l8faDeuwfv16vPvSrWiqI3nJOOeca0zEqZzFaXSKtDqilzMBsPE9W/xeJ1zQYqgGUydOxFsvv4b+ziEkUiX9P5UrSyA1X9JkKb591HysXrveAoL8nszjhwa8/mvbiK7o7Ihgyse1HL3UHuFYK9RrQwZEKAJXjLvDRcxMIBKpl0Rd69gOROobMHb8JD1TRnkGNCn8Mi8vmlQHTwApKTigQgiSRGct8PGzV8ceV37xboXfFGQo2eAwUsmEUSgrnGksYM1XSzB719lq9ISi9WL9BcN1OrLJpWAO6o8v/j0RG9Iu9cNjonzyCBGNt4KTTz8ds3beAddecaVaPcz3ypWiOCj8HIJ9eFHkKrgZQL63FmOZu9MKVM9W81YrWUbvn16Mo448Ct856iicc/75+Ot996Kcz1QxZtJ++TrSTc9QSYBpVhjsyPJGmRVfaBtEialZRjn39X+4WyfZNZf/DJSo4Jly3U23Ilip4Le/vkIpnzQdxZTLaT0QCSAHhg/kz/c9iKOPOgI7zJxp8nCKjGU89MST6Orqwbj2dpz4veME8w0lE3j1328iFh9Ge0sHXnv61wiHydGhAS5RlgyS8UEUWNw7iQ9PWxbtlTg5T66CPR9+sage3NKD1UtXYng4b2oGhYqieI66OJUaHHDgN5DKFEWVMJRsq8tHxaUaDEDqlejEM/KWWZ3bzyqldeKptqhNnpvXZf0XQ13kBysTtjAaGltQW9+AtnET0NTahqYx7ahXJCePxbrRfPaK2jqpnPY4i0zWQJrssmH66mnDSM7Z3lVL3leFYmmC5XBsibKoIx45WmQaMypifHNLi45NznWSBcYHTtzZi2G6cUhtDl4s8XHeAN5kX/VnCyWceNLJOPiQA/DTn5wjCI3TM2WnOssPmE0bpswmhNdmNLMCci4syjJyVD8v6bHcyYEA7rjnPiz6eBHuuevPuPDii3Hv3XdJY4XRSHUEu7KRWj0ULl5uUk70COWI1mLMmDbx6M3R2ei3cm8rF3H7ff9A1+bNuO7KS+QhSsTk1jvuxje+fggOPZC0W2q0WzdORSmvgc2XMnVlosjkaQKcRiqdVd5d18hOYxTPvPg6tnT3YnwHF/nxlrZVRnH/Aw8Lkz9x/rGIRpqw8Oz9lKOTt8OoXsomMRIfrqIorJmsGOfklM0FEBPnsyDpji4NH735Dnq7YoinykjnRjGSI4WB/PWAHC32nnsIunp7kU0ZYuFPUbvnRqEWJXab7rPPi03Sw4hipDD4Z+9pzNSJlGSE03qUipdLW+rqmmQhQ3GjtnETNfJX11CvnJyjeHxh4uuCDt1AjU4T1522moHu1FvrOa5PAQobV3yqFoO0QvKMcGarzWOgr7cbU6ZMRSsnNLzts8yzCNdYpPKOcfzTe0J6vxg2A5j+VIsfISKjOPGkU3DiCcfh2KOPdpxqi/TCN/Wn7UYdR1Sx4sNyeSc/Bz8fsWxGXUnckQzFE6FYQrECnHXuhbjiyivwm+uuwwP33mkqTVWXYMsxdZRrHM4UubjYlbvKJ5LjeyF1bFm4+kbYm+99hKeeewG33XSdToL/fvQZXn7tLfzmqkvFWZEyrkYBrX0vFp4b4WPAUGR3xCKeWKmsjRC++Mob6O4dwriOdpx0wnckabd42Up88MEi5cIXnX8WQjUBjCSGcMGZRyIaIneEdN4CKoUsUsSsR+LyMM2n81rkuUxaMO7I4JCIXUcd9x28/8476O2MYyRdxnCyhFwhgLwWBmG3IA445EgMxzIYGBiSxbyvf9REc2kGr5tcfgU2p0W+dZFXENEGI7ZulF+eipZD82T3Qq7Gf5J1PGUvKBbU1Iym5la0jG1HU9t4NLS2CW2xJqJZztiom/0eswPWWGTJ8rX4WQuymyft2elrBh2suO6rRRUuaC5ufiA+IP53LB5DY30denv7dKQzH9prr72qE/2avxRv2rjRvptl3TUbFvYejfwQviHEc+EHp5yK884+C4cccICaFVJKcovQdD5s87Dlzs0k//ogqqmMr+Q9qUqLSu5xnG4P4+yLf4F99tkHq1etwo2/vsK4027IlvWG5fusfW3aX//uvIx4+vBmMar7OoDFEUeuskXg55f+Gn+66Tfyu7ztzr+gs7sXv/v1LxAolxS1uYglr6aBi6LeR1NHjgtjebIdv5T24H//87mXsHFTN7bbbrI47yz+/v7YM4jFRjC+oxXzj/82giwiA2Fs6dyMww7dAYftP10AAYpZFLJxjMSGEBsawEgsqcDCpo6fF+Xs5G5774U1X65G7yBx+wBGclwURGhK8jJqaunA9O33xqbNm0U0E3eINRix3228gbiAC07wyD8zFZxucCNC/J7nveOaM3Iz+HHwxmveMPp6iNZbK7JAb24Zo0Xe2jFRi7yxuVWBhgFNp3itwddW4BqSwnPBzxcTHha1wTUtOVG1ad16BNat+ESYD3/QL0bKxKU54WfSBkEAACAASURBVOMGf/OZNLq7u7HfvHkSy+HuovmT7SCbnObKNMNTEWZtsr46M2n4LR8oKaynnXYmLvjpefjaPvsod1O+LhZfSTms/5IsBY9HHbscBTMHMWneuUaHx+R54Uw5uLA+WrQUT77wCg45YB8ce/S3zX8nHERZGuHmXe/nOYVMuPYv17qdDvZZtcFklUgkA2hqbMAlV92Ay35xMVobIrj0179D+9hWXHTO6W4hGLeG/J9MOlWliqo2cXIXPg3iJm5sbNbR/txrb+DLZauw84474fBD5mr+8e77HhRnfeFF5yBUyQsy5bUyxbrj3kfw59+fhwP2nYBCahC5ZD+yw3GpK9A+npMz6RQp0VQQy6OjvV205aFYGiNJqnsFxalnfcT0k8pXc+Z+G2vXb1Q32CNn4gxRd93fayd6qgaaNq8Vmepj+Ba6U7yikJOlex5OtNE7nnaS5nNiqgZaBFTnsV/R0NSCMeMmYfzUaWgd224Rv8aiPRe5cnFJhFhhy6EPuW8T5pTwkQVMThGVimn897XnEdi4+vOK2sNuvjOZSGhRbNq0CVOnTlGuPkpaZzqNdCaDvefORU9PNyZNmaoWs7eA5oI0nT3TotN8ZFVTxHI7XiAvfP73F+Daa6/GjjNnalJE7WfXovZHJKtuQVGu48lUyl7TpNiY9/tBay5IdlkZQVUHlMu45c57sdP2U7D3brNFTahTEUPusZG0yEnmB7Wq3JlC8YGqXWyL3Z9QHnfNplO47Po/4YcnHo8958zC5dfdiN9cfTlqqPNBVakQFyH7ByySihq04OloBVakOpzNa2UBRVSE7/f2x5/hw48/w35z98YRh30Nny9ZgZdeeVOQ32WXnKvCOZf3w96j+NO9D+IH8+dj3uwmHLBvEwrDvYj39Mv5jukNWZfpFCeLcujvG8ScObthS3c3EmmSskIochhFww1BFCv16Ji8ExrH7YS+/l6kEgktmnQiVm0A8lTW3K0DEDSZ79AUO6lcaqbFbh5BIm+5Z8ehDA8jSimtYpNeWhPyi2KXsxbNzS1obm1FS/tENLa1a5ETeeEGkGYkFzkjuQsYqh85PO7STyl8OadtwsErFn+Azz54m7orH1Qkz0xaq2uXirlGGmgpjzdf+zf23nuvKguRN3LGjJmor2swYpNbKJaXGZ7ivYNMitfayxbVzSHu+wsW4E9/uEURRgKgzPlU3HGz2YLn/3kjPGNNFyKpBubq3MXm2sz3o/QEtRt5fIv92NAgzJtUXU4x8RRg5c2Uq7ahUZuB9iDU6JNWCG2yHeZOnLy5ucmlZcxMvQqW5X5/e+RZJDNpfPfIb+HmO+7CLdf9SoxCwphMU7lA1MxhV4+dPIoKOekL2S46ajIXSYEipIEA3vn4c/x30Rc44vBDsP++e+Cevz6CLT0D+PpB+2G/vWZXfY6YlpHI9epb/9VC+Z+v74/GeuCbB4xBrncVksmCRHWoKJZJZJBIFjB9uxno7N4iFIVFf6imDrlyCEf+4KcINk6sSt8ZQmUDzjwR8ukRG9BOk1OTEF89leJJkNC64H3P58zQgEFASsNETTj5ROk3DWtwAsqisLaU80llJNdzVXORw9L8mRqpRTQ2N2NMxwTUN49Fx6SJ6r0wXeEaJQQqVQXJeRjOXsxnHS2aPRW6WocRjoaR6F6Pt197wajMm9csqTAfJz/FF0Xx4RiGBgbQ1tGKhkgUyZGEzKeMcG9FyKpVa7A7TWJrQuriGaTk4Rvbof7h+orcNM+DOPnUU/CXe+9Wx4tjdJRDIE2AXUehAxETHOL/VfRV5YuDKBMTV+RnemNT78zxeCMz6REz9uLmE62T6qf1CLCzmE/rVJIVtTjM9dWUhRu16sXuJ7ock9Vj/NXrK5axcs1KLFuxDp9+8RUuPudk3RsiNhx1UaNESlsWVfn7SpdIKnL/7c7waqH67seL8cbbi3Ds0f+DWTtuh5tv+4tqo6sv+5kKS3Fl1ISxFIEQXb6Qw0iC+i4l5ErAhrVfYN6uEzB9XA0yyTyy+SyaG+sxOJxCPFdBMdCE4WwIsQxwzXU3IEV1gUIWI0lSByh8ZF1CEqEyUlcw/kk2k1Z6EaPu+ogbDpEuT0Kfi1ApAwOLQE+m824ggmrlmEdD4Chqo6xVxIC3QpKMQ/4pHktE+Tf5+K1jx6FhTAfaxo1DXT17NNZY4wbyRSfXidr6Tpw1k00rYETDESTj/fjiv/9BV+dGy/3Xr/hMWoi8aatXr5YXOiO5xD9RRGNtXTXKqz2dz0t0f3BwGENDQ1i5eg2OPfbY6nGkPExNC5N+MJ8Y08lgtGPOxAGELz9dhGnTpmH72bPVTNnS1YUJEyZoKpsDCbzBvmPnoTF2QU3sxqKOQZ95DaxyEdAykFudN143moPWHKFrbEIt5TXccILwX2fZomaPYC9O8bDTGhV2yydmimBG+GGUYgc2nczyXXHVb2/D1w89ELOnd7BHbY2N2lrBj6pL/CYtWLfQrodpitFMDTmSmRGWrtqIF195HyefeAzCkTL+8vBzqA3W4JeXnIVoTY2aUnzIwsGr3pgs/PMo5UfRNTCIjz9bjk1bOnHIvLmYNW0SKqEw/vbIU9h5xnTsu++eWkgj2QzOOPs8tDaNRSIZRyFn+Td5NMxp/cAI7yUHqPnFwlzYP8EJar0XCgIAGDAioyV9Ni12MjY5laQpsoJIXHzexOp9CkoKCF+7rbVZEZ5BleCEGInhCJqaGtHc2oKmMR1o5P9byV9pRWODoSyM5FTv5WlpaFlFcLelwgx8tBIpYNmit7FqyWKEqPTKO7z883crxL3b2toUzdSlozgQlUZTSV0QHzx3IxePDh619m0XMz9iUbrb7nMwMpLUwqVlNQs7HS6eReiisnphTD0KOR2BpGxyATU2NSrNEKbuGhCGfRre6+SltIDYMvcFnJSpnIOzx6YpDMXX0QbI5Y0A5OQY6jm5pHx7a2vfXsuqdsGnDoLS1Lsrnu26oSFragKuXd+NRKwPE2g5KGZmAAVpZNtJx4FrQw6sOUQjAn0eaasENLtKHg3fd/nq9Xji+bdw5o9+gI8+XoTFX63GSfOPwcT2FnHPeQoYZyioWVned9Y73plh1dpOfLJ0hSbffzz/u2hsrJVg0f2Pv4DDD9wHkzpaxYYkX3/hFb82oaSiqQFI3kNpKusQjt+xtgjbkIMbvGaKZLJyWzevCHkOAmVUTmoBlzFayGhGl0FuhH+q2cdT12oF2bFkUwqQDJY0NhOUGAlj3LhxaG1pU0rZ0DoWDc0taGltE7dc00scllCT0g2IuEaTB01qa8rYtGEFvnj/XeQKtOi0/kxg3Vcfy8fTptUt4rCA4uJmGuAxSPMGCik/ZMHnSTvUGuHvbbfdVNx37734+mFfx55z99aH8ZFYPAXTQ6hCPKwBGE2JzvDh8+J5E/m6FKExFS/tQ5e2bDt9ZIgMj0lOM1nb2PGnWUjqQdlUvFrnqvKdsZXjwTNn58PzMKF191zL2bnQcdF7rUZKQDBS8HNLCk9T83wv24hGv2XXmFiNta1VGNF0VpQHZ7stJiQ95iVdpdqhfziJux98Bmf+eAHuu/9hFALADVddLLWC1Eha91eRTMQmMiQ5pJJTX4MI0OdLVmH1ph70dG/BhWf+EMViWhqJ9z32L5x9ynwUM3ENf5MQtvDy32oeks+Qm12TM3Tv2OZeKId2sm6+Rc77KYRLHG3i1GwRmrU66zTJUnO6SidrFqlUvDpCSE0eTkmJBarobikYT4Guzm7pvRCm5UnOzV/f3Iy28RM1CUTsnCiUKNBRcs7NPEDjfmpKWc+DIp/D3evw8btvIpPLGHeGkZ7/Ru6KLXIWQqYfwqOIaAVvJD+Mr2ZtuJdQjbkT89/Xr1+LnXbaSW/a0tSMeCyOZcu/wmGHH4bW1jFWGHLzcErcSQ0wEvGGcXcS27Tc2/I3/slFyi85szlTLEZE3mAxypWjWzvZzzZ6RpouKmhtX6k1Oc8d772jne0il7p4IqXFq61goyi46Xe36FVclRxH2ZG7rFll9UGYMFaOOSlxZVKObaxNprpOeZWLndGYrhfcvbaQbOSuUAJ+f99juPjCc/CH2+7GjjOm4oyTj7FNR3YhT9E80wrCuoZKGKRWJxWFx//1Nvr7+0UfuPyi05ArFWQD88f7H8fpxx+u+8w+AdOt83/2a10zrzOVHhGmPjQ06IwCDHfWfXaWjh5O1T1guinddDIdDdJlLq16RU1CCxL8rFHSQ9Jp1SEB0psLRTdaWTIELMiJsRSSyZjoxqRgcx1NmTQZ9a0t8i4lj4UyFAx4vIZIXdQGZxTNCSVWxOJk3ZIY7MKHb78pIVq56kWphkD6QxmBDSsWSXeFF82jy89zclqDf2ckzKaz1ZxS2iQakSsp1+SDFhgPYNWKlZgzZ45+b3BoEHvttbdGwrwZlj/+hVE7yJELmQvWoxu6eUXTgeGH9bwYcigYWYvOJMBj6aYNU1OVs7PFbkw5nULiPRvHwqby3XtpITtGoyu6NNDsFAnEtxGd1tIaXp9MnWCRmRs86Mb1mB7xAROoYUOIN99gLUuDPBdfn59Nt0itoDbrjldQCkTxu7sewkEHHIh3330Pv/jZmRg/tsnoCy4aiXBFDr/yXnteppwVxGPPvSlVATa6zj31eFQoqVsGHnvuZXzroLlSKBaSEQrg5DMuQjTa5PJka/cTe09nUi6NtEkif5/8RuZ9phyJGmlMJzniVst5SuP6iICnhpfJSGuaXvIhBbDPIhiSzbdcVvAiESj+POspBs+hwSEsW7YMO8zcHrN2203wIe3WW9vGVvn+7AiqZuIAM4NhqYTYYBfiAz34/NOPBXXLdVvdZsYX16hc/vk7WuTKv5wxLXeYGj4aYKWtXdoMQCO1YifaeJET/iFv12HstpttzM2nPjvP2lmiTkRSdIRX2/WmF27QY8WiujsOle+JQmk3j69fyGfNkcHh76au5qQxiLtGarXLCSXy5qlQc6/nFzsREKEfDtv1iAlvvvjYzNOlE27iSr74VfOo6KZPMjaVY6xMIxqxa8vo1VBXp6KIqQhTAW00R3flf/N60yMjaG5qVprAgorvkUcIN9z9BCoFNr+Aa35xph6StbSNr83fZUrHKOg7pqIQVML4++MvYjg2jD133R5HHHyg7lk8bgMbnK+kTAMjHn+P/z/j/CslmErvHg52MHAxdROd1hXuhmHbzxcKRuHwp6M2eNWShVJxlGS2DczC2/tPcSMSMeMC54gfVQR4TxqjUUVv8VzIj9I9T+vaPvvkUwWQ7590sqxdQnV1GNPSqsBaGB1FW2uLQBL2Dvo712OkrwvLV6xwi1qtLaVjJp3inFMo+GnwlD18NUPEL4emvC1X3So1Rh6zdd7SxhsvFPXAeWPJh5ZmuaA9G274atlX2GHHHVWczdppxyoq4gtHH8H9exiMab/PCXabsrEWv3IwZxTl0w6hGG4SRDef2hx1JovBit0zIH0uqZawo0f6RcxCRpvSFaOlUs4irorXgkGBJT5YRiPbmL6i5/uRKafF6OSWffS2BWKCqXwvPkQVpa7O8ASzdDGAm//ypASF5u0zB4fM2xVNDY0qxqxGss3um3ZWJ/D+ZLGhawCvv/OpFtNF552OaIBpTRp1dQ124hRzOnVld+gkto867hSZl4WDpqrABc5o7gldxLx1fcEa46BLKcEIcgxIHmrmQah6oY4ohqmmCTINhXVCMHCx3qKmIVM4aWaSuUq3EmYCZJXq3rL2s2dO0fw1a9egs7MbPzj1x2rzkzQnESHScyMBbFm3Gl2b1iIx2GewtuoeS5Woumu65TZ2p5SPi5wVtRfY9LRVfnhCeyomxEWxI4p/WjVrEgnEJX130Oe4fPA8jqwdXlYhwg7qySefjN7+XjVbDH82Apblt7Zw+H8VWeIc22khhIOfwQnxm4D+1krfQBzTv6a8mmcCKtK54Q4eMTxJvJ23URACNuQgBwtGcXu/YpEwobWOjdMTRiGX0g3lQuaiE8WYiA0XIZtWpIS66RwFC1mv2EnIn7eH4Rz13MCxwYhQNP79fU8jm0nh/DN+gEgNc1oyFCm4Sa615e7+tPWD3FxM7y9ajMXLNmFLdxcuOvd01IcK5gRirQKdMoWswXh+pLCIWvzoJ+dKOcxOrFEMDPTbyViy9FO1hdIic8G2wp6nOiG7sqjJbK5xc/Fz8Fr43HhfdPKpc2yMQ2t8FdXw489kCxktfHaQWeNFasJKUf395emycdNmfLlyJX581jno6BivgnTL+q+QGOhCd1eXGoBmp2Kbj3UYN1qEfzp5Zz9VFtiy7ouK8E1dnPFHCP4zT2LR44s0/oyPKL517cF/LxPBRUUclamF8lfBbx75oMaiQYy8iOnTZ1SPYf9z6o6qqeT80iXZZjwSFnV8bVJlRQtmdCttQw/mBJG43KaIalHdTSQ5PXBtEqYHLqeVYpebORRfw/2uT8WUB7PJ4Wicdn02xMtckxrY0uqLcIyO8m/0vDTNGl/Ic0P6KMx80jd2/OnDf0+VgNvvex4NtcDxRx6MhqZ61DuNeA4qqLilP1OtpWQeBeJ7Pf7CO2IN9g3249ILfmTOegGTBLH82fkD6bQqGISXyWHf/b+BufsdVOUX8XPp1CrYtJLvHmuDi9kXVABhfs+dyXvIFJHvJXDCpUI+K+D7qgZxY2j8PoMPoztfh89J3W03WkfmKU8gbq5iPoM1a1ZLWm/OnN0RiQSRGOzHQG+XcYvcpJGtTQMPqNNDeb4oXTTc8IidzhUEejYsqfg5R+5IXmCeTYJ8XhPSaWmxhJRj8gYr8kUi6Ovrw/hx41wlbsiDIrzcBqCOGLkI20Yfz1vnv5EaIAdgN8bkO3qWMlmxxiOOO96OSaN2MqIrbfF63BqVMbEfj2nzNfzm8Iq4OjkocO+c1HgnvKclF5rSHhWFjG5bG1EchNBcqRSZSCTLbW3MOP4MCzIxD0NGA/abSbUEMeKygxi5AKkA5YSMBMOytZTNoWsgjtowVXGbJdlABEGyacx1HbRrndqoJN7IvSmWyrjnkeeRjqeQyadw2c9+LDFSn3Z66QzPjPSEOfqwcjr/tPN+acWtqz8YGHidKkYJKTKV8BaTXrfFSXpbkWmFHdNVBkjCe6ybkiOUaq63iS1fl+hEjGjDNDU2mTa7z8lVl1kwZH1EWQuKyw73D2BL1yYJ9PNe+c9paZ655LEw1kQ+08Yg7R5tKstnBZLmWL+cEKLJL2hhFAsa+1f3aLTsuodW/HHB8GeY23Ez+NzM556UVuBuJL+Z8CE/GI9cz+aTfeKo5XRdXV3Yb7/9sHFzp8R/tMjc6JJPmq2TZrOktLeznNR4Jh7/5vFqTFpnC85ZUiebrB3P2oL2Lpo53Irdq7J30V6pCnkb1dPHYErbLAYF8oGrUHaICb9P6JDfox6hGiGjZBY2WmNJnBVzRfABgLm93WPX7nd+SWwQ+YYG39c2ic3dcspftF0e/64XMOpsEYORWtzz4L8QT6YwZ5cZOPob++n3xLWmNIYrfnUhbjLIlBAADodt7s3hkksu0ech4uGLWy5yLh4iRdYrcQuQMGioRpuA6AtTVdU64ZCmrBggdNoXijpF9f6yTOcaYCFu3U35UFGRzUVarZOGCFqjTRgc7Ed35wYM9nUpoPAeCo3j2nP0Dp92qRpzo3VUKWusiyIYsAAoGNQJUAWWLnqzIkacKzD5YSJSOw2aD6L7oCpIHb7rdy9Zid5bh5vERyg5/7pxKFObYuFkCA6LPF9M8r9XrF6Jgw8+WLsxHDI0weeAXPgsXGSfItlhm/lUfuogQqUwLvL63FxDrsK2Le3RrmYVz1EpFxm54UTU2gbvFlHM82Uc51u+lQ7REaadM+iLVFpuMPkpOZFLFlT8/Lw+GXqxgHZzmTqNuLGcmZiCStCoDqFQRH+X65sbVbMGFq1C/IS7wXN6Tm6xU9Pwr/98Q/Oi879zCCZPGKPra6ivk0S1IVcGJvj0wQrZCFZt2oL3PlqOxx97TMZnDGj+5CE6wufFRc7hC78xeb/4PT4HfpaWRoOZfR1lGjJW9PNzEj7ma3rZ6oaGOrteqiZ4141iQcQsiihtXL0auVQC6dSIUKatNAZzmbZT2ESL/HOtToxRuNRZUsrq0MG/ytdXLH6nwl3JD8bF7qOeuAjsTolfbR7wamZks9WFzQtuaW4W6M9/FzDvihceXb7SZqrh+Q28mdzF/qhj57C3rxezdpqFgaFB7LzLLghS09u1031B6iExFi/M6zgCpkKYEB4LI4cIidfuZg2NsG/pDQMzX4unCnNJU4i1NIsnhQpON3zB/F8b0pEJ7Pgz1SqOuPEvVrMQF6cDHjd4BHWKWIbMbDXCsiiqTS5yGKfuawQh+hqn2lhxkZA5K7F03m8uFp6qUv9yfB7qzPD+jWTKePyl9zGQSOLK876vMUVuPKEWgYCUqah+5XsFGu7Va5bwxqL1WLdpLQq5UXz87ruoRCifwXtgKV0ul9Ga4GYWf585vUPhGFhkne644GQn2sS8cYL4fS52Dmvw/nqdFcKESl8ZrOhiURcB1ds2rVyGro1r1eq3miLgjMycuKuMkE1BTTY3zmtVi16FZhnNkhm0k1qGwU4CWuUoO54qxvKEeizd4DFhqIbBc0wVKErPRdPeNhbxWExkHh43fuJH2K1DVVgc+gVu3TPrZHJnkhnX29uLMW1tiiD9fX06ish3Jvlm9uxdJVtBHoPNBnpHBZMslkWhsOOScbJ9O54Lm24GfMDUygtb04c3XItJNi5OeLRo42322iYRx1zXaAYcuLb8z980SwaJufJEsA6tNqE3uOKJx5RItFGKC5krh+BUeqBySoZIgE44I2px0fL1qn0AZ2VjHVKeRJbPKz10ilN+4/M+Mo3b0BPH6+8vQTwRw3WXnLZV5JM0g4JHRJjHmy2KpVRlbOoZxivvL5YeInnvv7vqCnz9m0c7IpqlV8PD5gfE3JyfMZGIm8ObdFtszpPBwX9+5d4MME4OgvfBK1nZprBOsuJEMIAZU7ZDLhPH6iVLsH71St0fUand85RLBdNbd2opVXVT/lU4U3RpdjdDqA0592bm4IQzpWJglO3AGy89Xpk+fTpWrVqlF50wYaLyVxGlHGmpWMgLA9f0DqMmAiJUyY/FLQaf40pGIBqRWDwLy1hsWMR2/p4WaamgSM7uakd7B4YG7GbygVKOgi3/yVOn6eaNmzDRLQorTNRMIqFp+Qpsv8MM+526ekM/nGybbrbT8ebxyiFlPhRi51sLSm6GrQ0wX6QwXbGc2vJRLSrHAecDshzSDfG62sAmmmxBexFU5b91nDu162LUl3SCxu62Gh6omaTcnxvAvu9zb3LdfQ3hO9Kim6qYNTPcV99fjOXrejGaT+GC074rSqo8Skm/lUAoj3zr9mpxVSq6vuff+BgrNm8RtDh3tx1x+P5744gjv4/mtjbRF0zuLy+qgHoOmYwUvrg++P66LvZFpFPDAXBrADF6MnBxU7PA5PcZNI1qTFFZQ6pmzdoevZ2d+OTDt5EcpuItTwoLZnp9l8owyFmt5ly71XQ05qY/aqmgNnZsCypl159xs5+e88TXDHStXSwI0SKvNV5MgIdQnkVEcQ1AYlYakyZMVNQn2iI1XOriOWRF8JaTmBDvOUCdRB5RbvAgGFBxwEjOn+VCb2wwTRfeQKY9zKfItDvowIPQO9AvtMEKSFOy4kPke5Nv0drSqmOTn5lIEFEOiY9yBpHv75wUfERmFLUGi2HD/BLLMko6MfN+m4DhZ2cdwdcl004R3M0OMiXQguGipH+7ok/JcHPVE9b8MTYfVaLMCUEYsNOt4Wvr5rsHqCPVTUfx+2aOZdLN/iGzFmE3l6/pU5e7HnoRg/Es9t51Bo44ZA9ZPpLiykUqgUxdX8H1B6BBkUSmjKdffU8qAMSmf372KQhWysiXR7Hg5HNEGFKgcPdGRL3RUd1X4vg+hVIN4VTUmHuTg+6LdQY0gRJMs4gkuSYZZw9m77IzNn75MZZ/uRTDQwNuiMQoFIIcCy4tVJS20cdqNOdYpfNWFboSHMXkcR0I1yh0VDk0ntrMAOQW+ecVLmjSV7u6thgRRlLO1K621rTfmXyQ4zo6qumFrAcjpkTa091tm8ulEuIXSFZsFB0d7diwYb3lpoQF6+sQGxxWpGcRwyjBiOxTDHYcecNWrVyL3XbfXdGnne/rFG0ZFQz6MqTCR/GIRtrIJ7dpEU4oeX6KR2b4GWwkzaA5fvFh8bMwQko70A1/cPMxv/dEtWpObnFEx6/SOtfUIaZuC5xpiEUtnQacpAyFMDw0jLa2MWqu8elq0typ0+rEcEeznWzW3RUW7FAf++wG8/J1b3/oJSRGsrhq4Rmo5C0QqSaqGgaHNMGlIoz5MgJ4+uWPsKm3R+nOvrvtgEP33cOYlnrPGiw441xjO4ZCVlS6Ti3HIsnNicdjxrQMBKrMQk9RVuvdMVp5X5i2+Q44f37f/eZh3Zcfo3v9KnR390gn3kYafXeVFpje5nYrDOzxfk44aJE7Z+5wJIhpkycgMFqQ1qZkSdyAuq9lBKNuXPmJG3+zdj4nQDS6JUkv9zDd+BqbGdyxGqgoFbFq5Uoxx3gTuZt9ZOToHBcmOTBaXDW8IWSHGSd6YHAALc2NGBoeVg4n598aE/ThB2UzSYsgHBJph1G9f2AQO+2441YHXnW5LA/nTeJRSYzVICtXpLmcmemCR0l8c4Q3jpMoflEaXGcQJcljvsPIPxmN+ftEk0xZ1qp7Ug2Y9nAjcMN4CNK38n0TSAVZBeraeRKYbTDr9vpFY2Qna1D5CM6GCL881YJ/D1EiryaAG+98AolcHtdd9EPj9ZDsJSYnmY5GRxaxTfckKibibQ++gGQ2g0CxgEvPP0U/Y1wUg/oaWsfjW9890bq9TgpEk2MOReFpGwlbv4RAA09znWxVEwYeuqaFbleKrQAAIABJREFU7um3mUIB++21B9avWoaVX3wiqRNuSNlWeoFXFxB0gjnBV4/hu5giT1IfyTmpP33aZARG2ccw5IrL1T5f2DrOHu4d2rKyQoomYRzyexVtXfNB3TweRemRanGmwsyJ1lin1ApBAfnlstAW/jwjBVMDIxTxoW2VemPEHNPWogK2rXWMFjud1QihsStKfQ56w8QTcZ0iW7Zs0bF73HHHIZZMCDXwVFCPSavx4KK7eVD7DWo5HTnMvhfgF7qnMnhsWqkCh4w56e1QGR/VGbUNFeIghokvMXVR1OV8o7wYoCkbDeuKy2EDzowmnHrxD41pEe81szDx6KWgayemv7/+M3HAl9/zXUV7yAEpXv3x/qeRHEnihkvP0ubRCJ4zD+Z7G5NzqxrYR5+vxH8+Wy4EZd89ZuKoww5yHW0rIP0Qxde/dRymz9y5unD5/mzfe2CCdAYO2jAYaEibdYKABfYJmkz7JGCUCvJrOPw+tGUd1i5bjM6NGyQapVOuWmQaDcCcNGyRKyq7ItxveEpr+7/X1UcweSJdnw0g8WneSy++hG8f+e3qqaYmY8/GLypijVE5NUSV2oTSD36PBYuGF5zln0FRxiNn1Nhu6nZSlFIu5nYSdz01+lhdc0KEu4mbxfJhw7j5YNvaWpSTc3KHBczg0JB0ERm9OQiRSCbEabBBBeNFMKrvudueeuC77rG7Lti7RFseaQvaD7radDkbOSVh6SLts/4Q4cFkxiyPJGJgHG/Db014lBuTKZBFZmuYiakZNSy4xIJS72mRmj49fqP4op1Rmr9DWQd+2cnh7Goq0KauBgnCmCK88T555MU8USlGb5GagWUU6VIYt/3lUbTUhbDw3AXVlJIomGqXoNUDPP6FqlTK+PNjL8vNgr6l1/7qPASDNhDMk0mwndr6Ja2B7//4XJQrtUKVvLjmQL/5bVK2bSQRA+cqeeTKiobOedGohjz0vINMPQKYuf1OyA4PY83SD7Fx40YnYGVQpg2X8ICxAOkRGn8yKBd3C15BlHWUc9ebMmUSRisFBFwur0YZYWQKqRLoYFAtuDlQLnJGcj3MfF6teEYH5qjSPXEjcSLWKOqYczMfMn+GI2z84tHPSKBCTJ0//pvRO/m7auNyAiVrtE0PJ3GhcbGT7MNCyBCGAlpa2CBI2s1X966gaELJsP+89RYuv/JKFWJMAZTLbjOLqVa5OqU2zqYbRENZFpYu9fJdTuW8VW1rJw/tbrra7jSnUkQxYpqc1NykDukLaoWX6CAXlIMDr59R2r8uvVG5wb2XqUVq6yJaGmIQZ5I0VNf1NajPHLFNcJSLvE6nhRh2gRos/moDnnr5HXzniAOx89SxQqY8NZf3i64RunZFxhqkcwXc9rdnFXEPnbc7Dtlvjnj+vEde60bNM++wHIjg8CNPEH/ETjxSKsqia1DGL5kYlqMyn7t6KWxaEcWKRHQy9/X244DDvoGWpihWfPw+1q1dqbxZ1GOHWinKVKzT6otLWxtuilwcFCv69YwE5ZUxc8Z2kqGjrQwZWgZ3GzLFe8gJohJTwYIhYoG1X75fIQpBbWy+J3NyLjAhHnoBI27xi+kHdwsbQuJ40BsoVCNuMNONwYEBcU1axzRLWH7SxAno7OyqylnwgXGuj5uBBYz58uT1gK2goJ1JGPHEsJoElJEmvso/x48brwtdv3a9CldG/v323Q8bNm2UZIbx2M0B2XyajCAm2Tspy1qE9jeRyIjQDi1ia1D4LupWixLeKD/44PjhUvUye3Zqv1hjyuHfnFvNZBAbHnZNJsqbmTWjInF1ONvuazXXdJ9LRzy7hT7qq5AKKJX0s7EiSyGIR55+BUvWdOGSc07GmDqTZ9CmCQRch5E2hmYLQ07SY0+/iJVbUpTExW9+eS6C5SxID+C/M4Iz+npSl/JrAHWtEzF3v4ORZ47PAjQ1ovu4ZeNG5DJJxAf7tIiGYzGlmPzsnL4v5AqonzARRx91DBa//xa2dG6U0xx1L/1ooBa1BKcsgvM9pRrgUphqurlN8U4HwJnbT0dTA6/LMVhFKjQilu/s0samQi/VGqsXAqu++I+2DZWWuLCJf6sACwRF8Bd9kuSbsHVF2V6XUhVHnKK0gTaIkTk0ix9SNg2C400LSauDFzFp0iQdV/X1tYKv/IX5zqj5C5XROmYM1qxaqVNFgwluV/Ok4YnT2tKifI353kB/v957n332xfTp05AjIoGKNAb5edQ0crWAF5nkgrNc1XNDyjYYK26EczN26q3K4au4tpGVchnORFqzgT5HvD5GZbXyS9YcE+FrtKJTRqmPclQW3TXaoEJUXITSyecGti233Cr0xOfC6XXDxf34XRE1FeAP9/0Tm3oGccuV56vwpcYkPwclJnjNRML4FaUlSWMzbr7778jky/K3/+aBeyklkltsVeOQqZItds1ThiIoVCrYdbd50inkZxiJD8lGJx4bQCmfQV/PFpeeOZFW6pjni9jc2Y0rfnM9Pl/0ITasXVkdKBevZpuikvfcBx2/HrY9VQWrOpQmWDOKHXacaWmlWQ/p9CbXitfgg5GN7bgT1qV8gXXL3pN0c5BE9+SIQHu/q3lUc2ZTuZ1DEDwJKZVIWn5b8Q0CqNo2SV3jmLDoMNqppThUxiWiwEYRdcGZprARtWH9eoO5XN7rtTS4q7mxpk2fhk3rN2pxjm1rU5OC/6bFWlODpUuX4oQTTkByJIXtd9hBRSGbObIrFP5skJ3NJ5ogvWZKSyRucTjbWSu604C/4/NCLlyxHl0Xt+I870k15aCxUpqSwYVU6NKJxC5xxIhIYsxpgNdSGS5AmbQ63XXee+lPOskKQ0QcehMISIfEw3JWTBZRWxPEr2+5HyO5Ai4/9/toaGjWfbAg5KjJHneuBLFmfSf++fL7qBkt4+qFP9YRr8UkvlBIea/nJYlIpf82G8NKIIKDDzkMQ4NxlAtpDPX3oS4axkDPFsQTZqXOYKN7G6zBpu4tmNDagb3n7YNNG9Zr5pKgga1KI8/pr+4eGxBs/Jrql2Mu8lnx/k2fMVlpiigCCkZbCXSia0glwKBk1j6+M0yWpuQrln/2hghapGgybeFNrqurVUHI/EZFm8OUycuojZhzFzW5iSRQ95AfnHChAfTB6kQNr4c3c/yE8doAfE0+eEYRcy4wCQw2hFhoUtTTTxt56irzblXwnDEk3dfNczJ6efiPBS7TkpWrVuGwww7DdjNnbG1juwfqh4oZBZSe6DXJxbGF4Qn+6qq6yG6Wh3YaFKWzmEchn3GtfagTqEXpoC1RCMIho5Jy6FsYug108EhVC5wX6b7C0WhVVsKKXQ6ZUCuGzTlbCFzwdsK2OEjQ3O+uuPk+NEXD+MnJ7HTaZJaaQCoMmX5xUIMO26O47cGnkUikcdQ35uHgfffSaczPxvdTEJIalY268X2NNuEL3xDWrVuHY445Bsl4TIM0lWJRuTm/KIXnkRk+W/7swQcfZP8Wi8uszMSLDIlS9K64lv02fqkqzpWbB7FizQas3NSJeDqHMxcchdnbT7ac3XbH1r2wDVnLj0Nq7pgFvAZU3CT/+q/elzGABNGYtKuzxtzLIhzb+aTO9vcPiFtSXx9FX28f2trahWw0NzdqCELcg2JBTRu7+Djq6xtVqU+eNEncFObbdioE1aHs7aUhasqiHfOzckE5LuvukRTnAe2Gc4Ewr1RzwikyMdprvIq880IRU6ZMwfDgkLD7gw49RIVnx7hx4l17gpIeasSIRbzXHvlgOsHFICivyo/wMnTWSKGqLAcKRkvUGbQIpiDAuU3XCeTJRHiTUZ6fu6W5pSr0yS6thg04OeO44iT68+dYx/hC1MOFagY5w1yNoVUqKvJ439ijuPOhf2Jc2xjsMWsaxra3V+dfPd+FfQ7e15FMEb/90/2yr7n8krMlMR1ATXV6Su9HeTUuMnnUc1C4RvMCEydOdB1gOx3o1KZ5WKJxgaB44x4tY6qzfPlyHHDggfqeBiDYH2AK5kyCfU3ERe4n+5uaGqRVaY3BID5evATPvP6RisZsPoUfHHk45u05XYtbHqvitGzjXeT4VVUxK7eR1MDLWT0V2LTyY9mO+2kfcsljQ4OaycymR9RW7+213IsRnQuNRWFyhBi2Da/yi5ujualJF86fYT7KHU7RIlbaHjYT/FiBSPV8aEkqORWLKq5oj80pf/4b83lyK/i5hoaH7Ca4gVjCbISIrAA2o11ClqW8WU1zJ3PBsVjddc6uVuAEyA3horSWv1E3baHzukQn4MNzmL9PV6pUW89hKeUwPNiv/DvsHBeYwtk0DSO/MeUi9axXqOhVo/SEn5EL0E+zC6v3cD5nEVnoUbrOQWks9vjzngjFnFyf1TH8xNHO5XVvaHlYzWndNBQFmsI1ATz3ykdYvGo9vnngXBw4dxf3eraZqaHO52qDKUHdM5+q8r08f8k3eoZSOTz57MtoCAex8/Sp2Hn7mRIKooHCyEhWpl6EEfk6PPX8iUBHPDajorUmEyfNw8ZGg1+d0zbTI270Ves24r7H/1ebg32TQw+ch+99c669Fkzck2mW7+76NIeGuls1dqzG4pfSrzVL3qswWnsykCQeaoIYGhyUKtLuu++BoaEBdSn5JHy6wYevvJfcDB7DIWvadHR06Fhh5JJgp5wXQk7ay+Ghkuqt16JjU2jDhg2YNHGioKkNGzcKZWG0b2po0JHHCySawx3fublTr0mOBiM1K3r50TMiRmp1ckjpCXas77333joteMLoCHYyxORI8LpV2JBA5EbtNJOaNdqxWuHu53nDNDRSpnd9AtnsiE4cy/ntJKBEhKZweM3SewlIUN+/h1AsYdH289WZUBn1mg0iPyPvKR+RDT/YQmeTxCMISnkqUBHLApvvz9fUCJsTexKnu1jC7Q8/L3OCheeeguYGk7AjfKp0VMZmBAgiqiH8e/sGld/wRtgq4qXX38Pazb3SqYnHkrjh6oVoaCBpLKAUhg0iIXC0CK83LrmCBQdLMjTCNVjTFMEooR1EhPooVem7ADKFMq66+V6leQxic3bZEeeccmR183NdcL7TD04wg7AmGi2BzFfWL3D+t1KgVV+8XRHpxg0RcKexQSFs201xixstO4uIEWmCPKqSQjpEaRQ2bvYpjM5KQUIhTJk61WQU2BSipUgDlXDLTrUpoLyVcCV/j+nG6hUrEWczqjaCPffaE++8/Ta22247DUETeuTCoKYhPxsZkGodu+FmG/YIK1Vgjt46xlAJE/vJY8eddkLbmDaURPc0X1BN9MsnyTqcfgBaMKlwfZM18DdUqEo+i8GBPjQ11iOfSamo9YhIvlhGe0f7Vgc5Z0/joUpufOnQCIYsyOpEtFHWIrIqlICLPXSHV0uIlMHFDSJ4mFOzi87lONoQrYowWT7PDm8RW7r78McHnsQ+u83CPrOmIlJLz/pGpTaK0s5ISt72TnhTC1+KB4Z/+yKYfz767GsYjKWEoPHz33LdpXKkszTZUi8jusHl+NajCLoBb9KUbULIcmVrIlqKTZTNrjuEy2/4i66BG2PihA5cu/DHsnlkjinBWTE2TU+nWg+5+2QnpZsHduOHgWWL/l1Rw8XhtnxzphrMywb7+/TGbWNaRGjfdipDrfJcHk3NDVocjKBs1jAn5a6X/qDr9vHCmMow4vImEwrkvxFtIVLCi6VEWOemzbrg9jGt6Ovv0w2ODcecYkAZU6dMtbZ+Y6M2CtOA1EgSiVjCiGW1Ef3M2nVr7MRhdCY8msno882bN094fg3hUDd/KA46WXNhavKZYqyPLHz/AocdnMiPupkl5q9GRe7t2uAMoazjW0+7PueEJ843I4t7eEo7XDDhScH74KkGfsSL127Qpp+7ZB8iYixCR332hDT9jGKP920aVYrJ4MLPKWXaSB3e//gz1IcDqAvT7pvCmmHpw4hPXx21s06xilANQzAHp9Q1ZZMtAPAZ/v3p1xFPJtDdtYUSS7jzhkurplweVSLtmKcgUxRfbHpOjzj1DCbsWbiFyHlintLGoqZ4UgG/vf1xXXMqk1Gaevs1P9XJRkKbBZWtdGX+nffTim3j1HDT+oEUyeB99v6LGprgN5kr8QMysvLPkURcC5Y2Hfw3LkYz0LKWMXOwzZ2bqkQn5mK8KYw+pjVu0/K8Qb7oEFkoGq02TPzPcXNEIxEMDhKLtQ+t+OBkkD1yUHTcGS4SPmDqhdTAkBcxC0tFsMs4ODhgC9xNp/Df+BkoQ0b/nmkzZ0qEk69BZwblyJTYUB5tE//WhbMZTx65emiaQzW222BPp9rSHePHKX9kJFaBpql8N5jhNF18p1WRzU3783UkuuRYj9pErhFUhRFFdnCQmXOm5nvIWcEJgDEF80c0768GxENBpDM51JGspkGGPIb6+qu8d0ZKGk8xvTBSmJkQsxi2Dq8RxbguPH3ir4++gsJoFv29A5g+Yxp+etr3qymJ7yb7mVaeCOqmcqLfbVrPHaJ1usfLCSSoCcbCXJNTAVx58wN6jlzkDEJ3/PZiTeITpZH3kCPm8T7onrkusrhCXofHDbXoxPv0nWcrHDrmMWPcZytwOjs7lTbwF9UciBiHQzJlxRKaWxqr8gpaYMGg8l4q3DIX5KJlOuM1x7UYyfFWzmZQITcEc2rPTWE+6QeobVEWFaFj8bjGwaRBEg4be9GZWhn8Z/ATM3Fj9xke7jtg3HyUjeDD5DV89dVXOPzwwzF58mTLGd1IGBemcVgMfVCjxEmd+QilFMNpsvC1rOp3Y2quPa374WiyGaZkzeYV6jFwNi7sgLcOrWz+QsbT8TRSO4rdwAAhSD4sF3l9rsuoyLTKNrdpuvjNyufBZ8DFKjTCj/Kxh5AaUfeSxDIb5g6LFsC1yN8xrhGlmu304f1458PF+HTpKqFejOYnHXs09txthyoi5YtMPg8VyNt8Vo/aVT+3S2994LNNZg0cpiJX3HAXiuWKFjnvx23XnKc1w0ESnbSuG6TvOcEkQc8KFtblNoDDvhdY+dnragZxITO0s4FDbnmKw6QUR3ewn+cbcBGRZ0KhRmpwcAFxMTHSU76CN2lwYLD64L3vO4vG/oF+0GuTd9MPWvDndaMpH/b/VHXmwXWW1xk/V4uRF1mWheVVYGMMGBzbCekESIb81TTT/9oO06YzZCZMOw2ZNjDMsJSAMWb3AqQsTaGlLQ1QlqZpO810OhlCmgRIYzazVMbGFrblRZIly7b2rfN7nvfcKy7DSLKuvvst73uW5zznOfPdbUSzMN+PjKI77iri0uUrnVhpqrLxVC7QRadRHZPueS6K0AQ2nLnkJp7R9YPnYfPymZ92dcWmz23U+9tXrrBkWdSJUsq/4clwo2PD9iqy6DQST9hjcM9I2rKLPNEYLzSXxbXhYBeWknve9Fzk1i6xIWETAA/mwjbdwIuc/6hjOIZ1N35KcPAzf2/i2WdJYL4/TdYSLPop2mhlYyLuoxGPTL8TL8li/MTj1DKYlExyTdr73Cv/Hcd7elXCHx0fi0fv3xL1M+POrwoPnnuQfKHkDOXCznAo/93FLyMgMhYzhHvz1SN7xz27YnCEgp6bpJ/ecYvgaU2HlkCU6QgilhXUPGdAkc9neBXRoD6Hyp7XfzwjZGEWJ9hDZU2H5Kaky8JFpuXUDimIg+K8+fPFYSGOExRXuks4BrE3cTgXzCLghAgLzPm1y+FC+Rwy6qXtS5QDgK4krIcbymQl1XFZ3DxYJhhoMnMRQGprXazuI8thmB6gxmyNVfHCEZdlfDzefeddYbsca/36y2JipswvZeKcqlMlsZo2WnP27GktGjxMFkzofk+rlPFiFlxYhOKJq4PfYUdO4JCQTtF65N8NOVoaO0M+9ZYmz33W2MGsiOSiyWQLQlV6sWpyF25ETyya0fAqrQilce8pjSYyFhmWFZQC2jHv+8Gz/6E4n+om57j97pvVUZQWHPhXa0IirfWRhS4bObcBZo6WkHPWJXIzay1AWXjkiTh8cqhM5quPR++9WUYDXRWFaikPUgpMRB8yLCAvkrVzhxYOk+l8lbf/5xWRu/igrGyqIFRguRSwZPESqvDKClt2bMAzATZT5iy3QhuTNwS0XS6Ov2HhcWyOlUw9/lZWplTf3nj99bj885u9YZrmajFRRQQJwDrzIPAaeBCSVYZ0EduSK7S1LZa668KS3Fp9IM8ZPXLj4HwW/O55TU1xYP8n8g6bNm2O40ePxiUbWOgmNUnGbaroweSUB9DaUlXTuSkhdHufNnGR9kiLzCLKvELWvlQw3RHjBnLumZCdUoziZ2Pqpk1YWsNeS265hCW5aeTFSrOFaLhDQzou9zk3XQqFskGzesriNbzphFtyGYiXjsK1MZJBRkhB6R9f/okSPEh4rNuHtt4UUxM2gDJ8WkMswkJeEwOUsjz33VylfK8TbMOLfM0WQa2nSsRPf/qr+NF/vaYiFffzBzvv8oTKVGgguRdEbM/u4pADwCz+6Z6PTkbXke6o7P7ZP89wkZ6+5gVA82ouaGLGHFzEDnbVcI4QGHZ14us5kxKLBQ6ayassVOMc03CVJEwKShwqLVwsFJqosfSrVq6wFFoRmOzr6RPMCIzIeDtx3Avcl4kkMTTJCgkO1AJdrFRgCU8WRnf3UVn0tB6cP3/Lw/PAXSvPsqBOD56ODZ/bEC2LFsWCZivOSmS/yEKkXILiXoUJ7iGkYJb02ZziLMtu92jR/dKvyCblGrNEzf1SbE5lUPqB5h1kKMQ1Oc9Ag6U2hykrfHkukmaWYkKD56sWFTKuO/kshIIYCCFBc+dFE+FRCYcSUVIxTaV3yzqQF+0/2BMv/ftPYmzEs4Ku++YfxYaLVgoRcd6jAYx6tpIuYdOgWCBZiHrNlXJoYoIWz0A5TxrXUoBT5bsuon/gbNz1wGNCSjifJx7dFvQ9aaw4z4KkW7wHIyoACRAGQWZmoB8WQgybRKoFb736groHCC9SVyPxzjwpY5vg5OcoTtMg14lJUToRy1S1bt5cxdM8JP4+kxd26eDAgGSCp2bsnq3z7YWSN5cQ5P86P1I83XO0W6zFpe3Ljfg0MRTJkGN/PxOGRxxDzCD53CRsnB1N4giycvrUoKwYMCKJLxY/4z9RY7WhQ/E5MCMblhtPiLR+/XqhP5w/1V+42ywEDXUt1ci0QFyLQqZSNbTsg0lU1nOUDpoeJm4b+C/du4bkFq69O2JgOLqCC89ntu4h1+pOIocXWYLPkNDimqbm4UEV9pReyVrV1L+vJmOK642sAMUKGZLl9tgYbq9gz0ol/uaZF6LryHFVswEKHn5gS8xMDet39jZUb2sCrgAEpu26YaO5xYk3LESe9+zFnd9zXhlezdTXx6137pTiAIv80V1bojI+UlVmEA1DOvXZ4kcYaI8yOuLCmNZD0V+pvPPzl2byJvFVY+OgLxb3k2L0xm/p5JhxkllE1MEuXVypq1os8639kivhQpubq+gM/4blt2inJ05Y9dU7HJ4IbpUKGq9MlvAGxJXcaLMiJ9UYTPEKV0iyjFU91d+vC2ahc8PFNy7KWJwrx6HETN8p17vhssvi0OHDVaTngz3vx1e/erWKOqvOO1/nRLKWMnbVhLAcM0MCFqHkz0rcqM0kuQnTaTMxTFddRYY01cEsvnzQhHFqTClQqe4DdAXOOakHZTyN4vwc2Z73fKZSUwcunsrQoJEgQZRlkhzGh81l/rlx+lyQFAIf2PF4DA6PR39/r3638/7bo6ECnbcofvHZRd0rDZeNF3ygBlEwDG02V9dEGoqMy+2tyNPrYnxqKm7b+nCMjLra+1cPb425mofmvIu4Pwt0OWGPMZXwlQR7Flr44Olh99S+8/MXZxSolxjaWWtttLM1P8w85Hu4KHxYjxokmkQh9cOqc9c9zcGlKgocxK7COi9saVHVkpiN+THwn4WtFjgJS0SDLNZEIZFm3PvYyUV3ccGNsmi5pLX2DbNEAnDomcFB3RxDSoYzz21fEv39A7Jv5AYUhVhE7nCa59L59LQWEcelUYMF1t7GOU/EuvWX2pKDW3OzC1E/3b0LRabSWh+lZjUzuc6NzzXlQiNhBsmwJXPLnYoyRcNRxY7RUSEPSYeFuZmQJJ5IECKsTklK27NosWlorgccYBQIiRyi1RiOysXg/zfMMUe+kZxpfpVchX7o1vt2xvjYZPQOnowLV18QN337WqNAkynGRJXVFWPoyzw7y5G4jG+Dad1ynl8TsnRFWsKMUHt/v9Gjzm+5e1cMFav88PZt0doEz8U5RCb8ivM12sXdU1yLKBPlntU1oP9zJipv/ewFjTjMcqgUQgt3mgeKBWJxEjNjXQg/hJVrRj2EIVcIscy4ebulUlAoo8bTgvA+mHxk6aAAiKtz0fAvcEFoCer7PIbGklCidhJrq251VIoOiYn7BrkQwwLp7+vTwiBR1eBZbozE488RuR5PBceG8Aa5DD63C+pA6+Lo7euLwVOn3Fg9MhIDJ/tj7dq1ml2D16hvrE2rEAU3Z3MmPVfum0wfT+LpGYQiiVZleFYN2zQg1kUTy+lxrZ60Nhvrz0LKbEQCCoSQIhVJSrhSULHahirMSgxP0SDMc8lQwaO8/XlqpAB21XABOELjcec9O/S8zpwZjO9e/2ex/sKV3lRSIDOsR+xuL+RFC2SbCFQqh1XDU62xVAarVZidK5EHTcet2x6OM8Nw/idi+31borUJDnDhkxeuiwzDxLSluOtNGebvZbzG0HKclLGqvP2aFzkxDDuNrywaMleosm58cGkX3oUUnvR7XFWjUA8sF4ufjcCrHWWskyerrpedlbFoTtJN7ZBsQGVxJ3WTG6CZnSUEwTojW5bFnEQOUonL1qBOYdSJE8ej90SP0BJweQvkz9F0B8IUeBfE9nT0yBOhKVimIjTOcbFhUVEuUJII4aqxMboPH46WlkXx+S9e7nBBnGsTwbg35CjwKDLJ81x6L8DE1Vk83F/NwCxTJKR5s8CPOYewAAARqUlEQVT6M9wjy+5VlISmS+eYRhC8WTRFujQb8B2eMi0h15sKvLaQjlV5kaBhmKhYpyGycle2oFlGD8+HeD9Mj7ff74x/+dF/xmnYhmNT8bdP7oyZyXEZKnoLVM1mo6JdoM1tZCgT0BK0VsM1hUllkXLOuekTppZBrGuIh3Y9Hod67bHu/97N0dqKd7AXVbRR1hTXJ1kSkmC04AsSxc/0Oxzr6cOSP6+yfsKCTjJ9Cz1hzRRGfV8SKFwihRVZUjU2G+pRIaivTzuckIWL0Fjpc0BXEH8ELoJvciYWt7VpUyRKIRdepjhk8pX6JuJSTNVUvji7lAvDWkiOoTQOiG45YVEhHjifQ3iSY2C4VjYt1pxFi8afj2cxHNUMuNENDXHi+PHqAiUE+vjjffG1r/9OLG5tlZbj1AxkpqJgq9Co5sUyVMoFTm7AvyGyxCACPWyJBRHv1z4/DYwhuVoyVvO2bhSXJRTb0iAOz408KQtFHEe48bjDCLfceTE7BGWxwxBNnfGiXlDx9TAArLFhbjz7/MvxUefB6D9zSoKmj++8R51FvKTZXgaVEe7yIajwZjiUi7hWbCgCQAU+/UzYVDaxWx4r8dyL/xpvvveJwqvbb7w+2lqZ3OxOoXzpGqHoqu3LnzspLsuYimdDIxNigcqS58nY9eYIQHOuiRfBTan+Yf3ci2kp3WpSqrEkxit5yYWpSINmiLvOQQzEsmPzaHDUqBsAMikqXdz8fYoDpVtlIacKbMJPeoCSiLA10AhBBEeLbjp/A5bOi+/RCFFvqgRDK5akK5CcLKVK+G5MGB4+K+vODWWYkxLtIUst4EpBYI4dOxbrN1xm0pWaTuC1JL7tEMWS04WzLuKXawjZIpg8DFl44K8yaItcBbK5mnzL6JVsfK55CrPw8CjJ++b6OU9tWFnJWsijzVYQLYd9bqY2EpMol+nEeq+8xlQ8/PgzcbJ/QEjal6/8QnzrG3+oiIbzoDosSHDC4aQaT6pjJXmTNzLX0VgEn/iZZ6EcqIAKuf4c7hhQeG/PR/HDf3tVIfKN138rLl7drk4fRxqO4eWhyoAuN8Eg/WFNd3pNT4+Mx6uv/TIqe375smF0Nfz6w7lIYlIYgrg2YnMLyLuVi1finQk3EjrQCgUGjoWmCKTBUhMTRkpOnapiz6IMSHfD1gpMmvCGYg7JYVoqFhUPIXkIvJfBprzHHgBejUdWszl5wDmZwe6Pm1JGrpTN5CR6TixdtizeePNNdb+w+NkIlLatqmWvgWUcHXIDCNeEQsC6C9bqHlGs4m/XrFktWNUu2A8/q59GjJwoJY0XaEDDtKRQllIapXxfprw5kbc3TXpAWv4sOiWakjlBHi/DnkEpobnCmkUYQss8Tm1GlIf5ikiFBy5a71hNznvb9sdjYAD+/Ej89WM7onF6PMbFxDRKI4FR6bx4XSD/jEG0qlVJcAtPR1QInkthEqYHzXOqJsyVSnR1HYpdf/eiPPCffvMbcfmlqxV6sejF0ymficy3jaeFSIF6LXMxHYPDY4rrK2+/9rxUd1w6dmiCpUmcm39nB2Exsr2O92X5XoSuQhDSDJgyuQ1LRuKHRcRiLF+2XDrkubiN61oISN3WBetVowEioqV6OFsAKHkeziGcoPH3wIrgyNxAHgYJH6EIirqESRCxMCpUR9k0eIXWNsZZL1DY1dV1UMdYtLBF8a00xieAzPoVErQvXRpHu7v1u46Vq/TeAwc+0QhyEtuVHR2xdMVyyUfkK2NNhy01TUa/x8iH5OeqtFrHmbWma4d72RGaoYs9pammjtVdNc35qpncJb1V6EL2sBbrp0nWiDiV2UZO2k0fADwwAS2ka3PvjifVIM7n3bvllmg+pzHmIglRpODwRtx3WfOoqPEl0ZL8Oi0hJ0OT+grxq/B/8loyzq6ibXV1cdPdO7XIf+93vx5fu/qLWsgaNlYMnBA0eT8MZgEf4P9PCSiLgTMj0TtwOiofvP7KTHaL+wHNxOLFbbKscDLMObB7kGyzhriWsSbSOTQMSKwN0zB16TiZRa2LdBy42rzPsbN5JlhOD0pltMb8Iq/22XiLG6AumUK0MkznRS32orgfdOzbimYIk7AV500CnTqHq1Z1RGdnp8INrouQg3PngSOqRIcSuuiw8xDX50EQZnFcN2SMK05n0asNK2GrsTFJaYDC0NShToLSECy8WTmK+eXkFhnCcFli/zk4rS5eJ1duqK5tGn40ZKfEtHw+Fi29GhvapXQP5sr7gLVPDUaHm6k0RjWbyqMEO5wDpIWso6H4UDz1989LmgSC3R1/+efqFVVFs/DuZQSnrRdJc4z6VznvwosHs86NR0TgxV6ToqivsxCUOp+KWKm91HTcfvfOGBofj6u/8uX4g9++qgpypCARn53sS+BCjqtZSzPc74jh0ck48OmnUXnvFy/pVma5226InYY+iWNLYi0qcE5kDNCroVR0UIP0mR2n5Bg/J086y9petHBCjJ/nBjJ640pokqyqu14uFwycVjtCl9KVXlrXCGXo3OfFA6PsXCWJ1dUL1ycZJpZjIYsnD9MReYu2Ni16qqSewGBYcv48q4UtX7Ys9u3bp2tsnjffClWNDUIWkO9YusSDwVjwXZ8cFLFs1fnnRZsGCOTyzNlD9pachx6G3mAXS/KucGaWFEZSIBSf2+fpq5ESw6X8RousnPds78F7Cc14U2LRqJ3lpuA5Z5hgUMEd+xkr82z/4bmXYs9HB7TRb7jhhtiwflXU5+DcUYd4arYWMat4MVr4JOfmn424OAlmkWfrni8K7+XYXAl84YaLdTkxEbdt3RFnR8di/cUXxXeu/f0y2IzNz3Axh3uWJZxWglnziuQYDQER7cTJ/qjs3f1jayFW4RmyZiy1yf1CXiQwhEv0AsvqFAdvaWnWourt7XPi0VCvEABXr+aVKayFS/KgHA6JZqohhrDRErbMhpT8kLzwkPk9//w1skZr1qyJT48ciS9s3qR5NyuXLxVHJRMmjXcZHpEqF7g2m4ONwDkDGZI8o96FbAQ5A8cknOns3BsdHSvEW+k6eFCV03PPbYvdu3erGMUmJx7kfHJ25dq1F8TBg10KW8Dd93XuVfvelVdcEavXrI5GkILSqZ5ldsGAhTRGb2bGzdqkEkTKwV+lQlo6+1kMmdgjLZohW7r9nI/kceew+TxQKgtI/DuTilkYqVzMprUxs7fmBf884/1tOx6LE70DUkh46rFHolIp+imFm87UOiw/BSlosaJ9lIpjts55DXkGaOZzCp9K+Jv5izhEqsi64APr9K5tD0TP6bHoWLosbvzOHwumNAxbJoEIdvU4+fROGEHicX6Gt3J2dJyKJzE5m6D2wcQzCNyDQHh3+QZjGSTQT7tYSQhNjmLhe2wISQfdOMyMobIpHRFEfDRDyFDlbPqrXarH1SX2mckvYQqhFJsIKIxjzm9eqMro4UOH4sSxo7rA9qXt1Zge+zE0MloYeK6AJR5O6OJN52YN5hQRToGtt7Whob4/Ojo61JBNzNy2uE39palnqFh/0SKNgHFDd5OKSd2Hj4ofkxDqW7t3xyUXXRybNm+OxrlWpeVhzE6wsIC5yBMDV7xeQaICCylgzAtb32eoAguRBooyMKu4f92/Mo5Elr1UktO6SQO8JII2LNagVCEpJ1EI27f0A5vk1q0PxsCZIQ1K+/79d1W1WSQnYR9URtgw2jLntRqpMXzsTi0suCICdWJVDW4tjEk9FjW7+D4RAt1x931xYmA0WubNjXvu/IuozBBJTFjOoozCYb51Mj0xEHwAuSfeh57bwaGRqLz7ixd0N61JVxcrVqyUxoqtaBn1XU6QAg3jSdKleXES+xFn18YP4kqwlBR3QCVYpFw0Av5wRJw0mZWWYQm/T0uVMRwbgsXEezhme/uS6D1+TIKfyEF82NkZF667UC1zX7riS7GkfZlCAZeTGbdXH83ooJ88WR2iJUk7uDJDwyL88LlCe6CGskEpEs2fF+vWrYvf/O9vFHcT8rB5IYYRMnF8W/wubdoTx45V6wq8F6uOyM6GSy8TD2Pt6vNiskyEZnFxr9NysiCTXelNXvRvmjg3L6VMzmyMvAAUrpTGkVoY499nl4x05Kem5FXxrk5UiyY6c0c1tcOdWWmgqt6ifk7ccNsW6Rquv/Di+O63r1V3vz2s4+wq4iM5PYcmRQJImR+LWiPJxTyke6xWzHGiaeM2+/zze57j0888G7/e0xkxNRFPPHinvAzXntZfFn/SSbgoIOIpUrtwbjcyORXHjvZE5f1fvSQ7gaVkYcj9TSEV0Rq9Pb3VCh5hCskYNz5RjoSEHMYwfqQ0HWYSMTUpHgThAjcl40CjJ97xuYixgqllbkvjjnmSTB4SoQchRV3pfiEbIKPfuHGjijSEFufMtcwF58oNGBsfVZWWG0NIsrdzr9iSoCuU99mI3d1HVDDiASxY2KwGaqqviidp5iihTooiwZZUY/ZCxm7P0waiwsomOTVgVSkWFB6M9r+VKzqi6+A+qRGs6FhVxqDXFKV4P7hwCsZn2R7dFM8vZR59rYsmjYJmVJYxirWiixd5VhTFhFT7njkx3Jts2FBoUKivfCZWXVXKMrVvz4cfx1P/9KJkJB7ZsT3mNVh8VLWCkrjizXO0etW6l7GNdD9kLybGI/+OBaq8T932OXDWtZl8pWfbu78rvv/k08pGnnzwjmrcXrXkolVYudYgBF+Z82QaJYZlGAjxgzde1syg9iXLSoKGdJgnPvBGNx64QpbV0IzZIDZZjNI4acpRQE9NTgqkLfdcEvuZUO/Yz2V2FrGLPiSl5q3wcLkZfGbKGOfDRZZX3fd9FkCiCCMJaZGWJstYFLPR+FxCFTbniuUrFHrIRdOEMcHYQFd0JSTaukiIAAkl6MvRY0cVbsGF5zqBKInz5y+wpDXYvoa84tonJ7VxwJO5R5s2bYruY0dj4+bN8cG778fhTw/EV666SuqwF62/RLDXbITDpXrHor43uN3CFiRWzxHiRbo543jLgTjurmLQs2SPEwnTSJGikQga5SG67l9NWoLi87ocRFsfP3z+lfj1B3tjcnw0Ht11b8zjmRSqbDZ5cAwMDbF4IjzVZLZYaBkLzWB1cQoPxnu4VqsJezZTehlbeDeLnx0ejc79+6Ov70xcueG8qJvT5AacOWi6+DjCzsvUa0AR4nD+5+BDFOPYysTklN2TFCVwXwqq1rX2rnJo4VjL7VnZY+mYl8FSbqL1Q8JS2dIosy7d6RwPCBFqbMb4Hi0+12623HzFc4VZlzs/3SQ/s3BBSDgnFghdPjltjmMjpZxkLaEfpSjChkV75cDBA1VOCfCVuBfEj+VawP3T++QCSeyexNXok72N6AP1DbLooDFsJCw5OimMf2lZvCTefOON6Os5Ftdcc40KbEjstZ3bJgpqJue+d6bl5n3URpguSrAimNFcXXByvX/2oCj+vWjKSL/FCT5GLcOcVO9lI+agL4UdEh1lwh+qX0aW7n/oseju6VFxb/u270WlAvhs66yQglCziDglykY4m4u0irYIEbLBURJavur5ChlxmJxl+QynZvPgxeqcmYwB1MJQ5sqYn6IaY2KE66dU91SMjE+ol3h4dFysysqHb74i7gq8kYyLU3SdpI8YlA+usRQtIJOhh8UsLR6ZDQk5Mts71ZMM8qaqAF4qgCnrlfi2iVfuneQ2Yl1YxEg+w/dgF/MzVpvw5MSJnuqxchOA1UMVxroI2io9k1hv+NJYHpX7y0wisF2sM+e/kOZn8TKca0APxoKD8+OZstLqCqzVaU/2nVR+QLLKz+DsqerFZmma2xxnhs/G8SOHhKM3L2yJVaA1DXXR3nF+1YhIqF8JamH2FTgtUa+ysqoEK89KcpHJm7iGytgoWT9F47AKdi2R/8JL53gyVoL2Epo0LQXPcdMtW6Qp/ifXXRe/tfEibahq0a4ImzLYCksqmkaZOwRfCLSlhgT52BmO6PtZn5mKBYk+JYzoIpo9m0Y3MhVD54/C2bCQLudfNLYjpGrFLtAsdQqhqDU+HQsWtsT/A30+euoe8TOmAAAAAElFTkSuQmCC"/>
+        <xdr:cNvPr id="1035" name="AutoShape 11" descr="data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAALkAAACLCAYAAAA9Hzj6AAAgAElEQVR4Xmx9CZhdVZX1usObp5rnTCQkgSQkEEBmlVGRQUFRnG3axu62pf3bEbUdsdV2Fgf8UXGeAEVFEZAhjAECSUgCJCFjpSqp1Pzm6d7/W3uf86rwt74vXyWVV+/de+4+e6+99tr7OH/97vXhRKmChatfhkYQYuzoFKq1EprNEImYj0TEx/TMLDq7ujBbKOI/v/4VLFq/Cv3HrUDP4ELU6zVUSkU4QR212TwmpiYR7VuCdDyNTCaFnu4+PPHgXTjj9LMQyQ1geHICSzr74DabKD2/E0///g/46Ec/iqVLlyKdyWDDgw9i4ZIh1Mp1PLxtD3LHnQg3dBACKJVLKM7m0d3dDdd14fBPs451/W2YKpWxe3QKZ65bhQ1bd8B1gV//+EfYu3M7ENYRhg4ajQaajQCxWAx+LIZ4OolYIg4/lsA7T+zC4u4MugeGUAvqKJfKWHTsiUjm+uF5LpphiGaziTDklQBB0JR/+34EYbOJIAgAhPL/vu+h3mgAYSif6XoewrAJ3/Xkuhv1OoqlEjzXhec7fJn8XjQaRa1Wk/etlsvwPA/NZkM+3/d9eU2j0ZR/RyJR+cxm0ITnQj6HV8b3b8p9NuF7nryGv8fv0VgE9Xpd/u44+jvRSBRNXnsYynXm83mkUklUKmU4joN0Oq3r1mzK7yYSCfkMXk+lUpF75b/5f/ZzAEd+l/cSiUTgOY68lvfDn5fLZWSzObkGXksQcN0CubdEIq731WzKOuv7VBCPx+XfsvrmWvmMItEIgmYTjuPK/zZqdbkffm5o3sd5y1uuCPs7snjzVW+A6/nwIwlEkmmcc955eOXZp+OUNcejUi5iwcKFiERjuPZzn8Xa885AYmgA/YsWwwFQnJ2F5wQYHx5GpVZDbsEypJJZRONxRPwIHrvvzzj7rHPQObgSR6sllItleLUaGhufxYJkHCeccALuv+8+/O9Xv4LCzCwuvvQ1WHXyyXhhdArv/fj/ACE/RRcEQSCLxQfCBYj5HlKVGUyXq6i6UZy0ahme3LYTIQI88cB9eOiBu+GhiWYAWbigGcLnwkcjiCUTSKXT8H0HH3nlQhRLFVTDECesW4uDw4ew+qSz4cU6EIn4cDzXGIcrD52GxofD9+RDdF0PjWZNrpNPQl/jIQjVgPgM6tWaXDPvplKtmg1Bw/TFIPjF35HfazTkPeCEYrRBGCIWjcpD5kOtVmvcUoj4PjzfFcPhtfC9M9ksmrU6LUReW2+oASKkQQVIpVNilJ7nG0MLW5ujVq/L5wTclL7dJLoJueGaTd00spmaDdmYvBYaJ/8vGo1gdjbf2hT8N4JQjI7Gz7XkvXLtqtWKvFcu1yZOgxuB76t2rM6E68ofcROoIesXX8d14uv0D52MI9cua+w46pS4oS964xVhOhrHe666DP39/ZiZnkV7Tx8uuPg1qDebOH7pQpyybjUWDPQhnWvHdZ/7HJadsR5ebyfWvuw0lColVIslOEETB/e8iK5sG6p+FNGOXvgO0JbJ4omH78epJ5+M7mPWolCrYaZYwNGjR9H37IuojE/gTVddga998zv40x9/Jw/l2WeegJdIYvfOnQhXXoAQ9HbcrY54KFpRJOLKQ/YAtLuBLFy+XkMkFsNMqYS4F8HBfS/iVz/6HuA6CJvqHbggfB83QiNPIplOiZdY0RnFm08/RjzUwLHLMPziPixcfiJi6R64UV+8sPUw9gGI9zQPPxaLo1apyrXROKrVKhrGCGRzNgPZmEGzIa/xjGfm6/iZ3AjcEPow9SHJ5wSBGGQk6sva8LX8Nw1KokKjjkaziUQ8jlqtDscJ5L35vnKfZtPRu7lcv6CJeEy9peu5cB1XDYRetdnE0fFxjXT00I4r7xOLx2RDAIH8nJfF9baeWiMaIw2vXz+Q/+Y18jXpZFLex49GxTnYe+Nr+fdCIS+vpxEzKuoG0mjDTaRRUvy6vJ/L5xmGrcjAzy+VihKB7OfyNfw579s584orwngkjg+9+RJ0dnbA96LwEilcfuWVqNbqCBtVrDt+Jc4782USmr/041uQXbYAYSaJNeecDcd3BUJkEwns2bUTC3r6sHN4FO2Lj4ETBBjo68eWjQ/j5HUnoG/pWkyU1Mg9x4W/4wXsuvtv+K/r/gPfvun/4tZbb5WbvudPv8dVb3krpqYn8fvtU6j5UThmx7pBKDueN2S/6pUCGnV96H2dGYxMTiMZiaFcmMZ3vvw5432a4hn5IGlsXiSCqDHyZCKFTq+K/7z0RMRjMQytOBa7t7+AoWVrxcidiCfeSIwRECPjl/XWAknobgJ6OGcODjQbAk0IXcKGblIaAkMsf86Iwt+zmyca8VGtVeV9raE7oUYgj5dA6AGgVq0KXKExibG6aoz0jrF4xHjtUK4zlUy2rpMOgh6Vm4/xRCKFvotEAG4W6wGj5nU0NoE9svkgnpje1cIeenPahb1v/pzGSsehHruJZp2G64Cmyp9zo5TLFbmvWo2bUb1yNptF0OBzqrfWmM6jWCzK/ytYofHyM32BTnbtTQDQe/XVIRD+CKw958rXh64XwweuuhDZTAbZbBtCP4bb//gH/PBHt8jNe16At7z2NWhLJPH7Rx6G09uBiUIBi89Yj5CLUamiu70du59/DoNdPbjnoYdx8kWvRqlYQm9nN0b27sSCrk6sPf2VGJmpoFAtY3psAgsqFbz4l7vwr9e8Cz/91W/wo1t+Jjf+1IYHcP6rX40QTfx0416UYyl4TQ1LXghs2bIV69efpBAmDJEvzshD58JFfMANPUQ9D4kI8KX//pDg6TBQXMmbF1gQjSGWSiKRSiISS6LNqeD6K0+RBzpIT75nPwaWrkE83YMGH65Lj6dGJR7HRAQbKvnziBcxsIPRQkOqPGT+TqC/SwNnHkMDoCHNzs4imUwa7Mz/p6fWTSOwQHApMa+Gdv6hQUdjMbkXPny+nh6SDzUaUzggkM51EeH/1whNNLoIrjdhnJuP3p1Y3WJgXot6Ul0nzQM0v6jVqy2Yxvfjz2m0fC2Nn5tMN57COG4YbqpaRa/d8yMmWjH/iMjr7CbV9fJQKZVMblKX97T5gPX+1qj5vup01HHQyPn7xWJBIhHXjGtP+OW8+uq3h44b4oITV+DUtWvg+XE0PRepbAaXX3KJ/GIQNnD+Oadj6cIBzNYa+MvzW1Cp17Ds9NOQRwNtbW0oFQtIehGEhSIevv8hrL74YoSuh46OLklII/US+oaWAZk2lJohijNTWLNkGR789Gfx6Q9+ALfe8Ufc8MUvi5dmRGD0cBIR/PL+bSikeqA+TBd900OP4vRzzjSOPJQkkQlHJKaelp4p6vtwG01883MfQcBQTE9qIIuE8VgEbjSCdCYnDyrlBnjby7rFmBctWYJatY7B5euQ6RgwiZE+ONkgkhBqAsgHRaPlYltII+EUQSshEq9sjIUPRDwREyPZfIE8CDECwg++r4BQhVd8+GpEUXmYlUpVkkGBSUFdjE+MPhoTjKteNIZ6vSqYXD6Xm4bJsxh3aJI1hSj07rx/xf9AtVJGPBEX2EEHx1Wnd6ZBEffzJ/wMJqaZTNrAB9cko5pPlEolBA29T143r4fPldcuUDMWFe/PLxorDZ3em+/L6yD08Gh3zaYYPK/FJt9cS4nIQShRwCakAma4WAx9IWQtEomkOqMjE5PCXTSCKuJgtu6iWilIrvfYoxtRnjqMZ7dtRcRhiHAQT2Rw29YnUKk3cPyZZ2Kiyd3t6cIws80XcGDXbnQtX4VaMoFYNCHQonRoPxatOAE1L4bZZgPxmI9kPI2Rn/4SX7v+47jpezfjC1/5smT31VIR2WQU6c4O3H7PYxhLLkLgaMLDr+LYBJJdnSakA2GtKtg1dEwSwhsOQkQd4Ltf/DiqjbpACWvksiARH34ihngyhVQijrjr4RNvWCcQK9vWhoMHhnH8KS9Hun2glYCp16D30cVXmKHJnEAMYVYi8sC40kz4aICEQPx8xfCKa/nQ6UnpIPgwbcLH95eQzzjWbIiX5hcTu3y+ID8T/F+rolotI5vLoZC33gsoFkstz8aNFCG0aDSQTCYEY4uXZvJuYBITYEYU5jeEMPTW1svyPrjk/Dfvk/ekWFmTZ9fT9eC9KFOiCSbtwSdMkIRcI5IaJkkDXxwWPa4a6FySyNfyveiJufn5x8JC+ZmJZIxUNpJyE/F3NJKQVWEkrAlk4cWLowit5Qhi0i/ChInhfdj04J9QKx2WB8qL5A3EEwl8/Y67sHt6Bj2LliK7cBDFZk08ZcKPoloowWvWMT5ZQK2/R3BTMh7H9J7dOPWsc9Hwo2jEkxg5chh9pAL3D+Oa40/BX/76F5x51jlYu3Yt3KCB/fv3YdUJa/HgE09jp98PxzADfFCB4wF8AOTOuNj0ULUK4CptFAT0Sg4ivocbb/go3KbSSpLANDT59KMR+LEo4umUwIWo4+Ctp/biuKWLBcaMjU9gxZqTEUv2InAB31WPQwO1WJafw0inibDmDYQfwrQ0FCJEIp4YsKv7UxZdvZPwJAotJEnT8G4pQBq5sg9zzAJ/j8akhk+zVCxtowtZDn7pJqQ3r8GPaMIsmJsenQZKGEMKsKpshvXafB3pOkIhvo5Q0CZ6rQ1ukvdqTZkiZVf4Psp0xGJMLn3MTE2K99VrdmTzM/HUtWmYqEN8rYl1e3ubrIF1EIww3HyFQsH8vhqxpRyz2Yxet+QJ+mx4rfx8uzn5f/KaOSNv2Ti2bXoIh597QPhywhAJ/9EIIn4U6XgSM1MzmE5m8M277kf/mlUo1Kqy+2hATiOAHzYwumcY4dIlsrMy2RzGd+/EKy+6BFue34Wh41bh4MghdORyaEwVcNXgMrj5Au666y/4zKc/LSHnc5/9LM4/7wI8/czT6L7oXUConmBB0MBEqYpCPAnH9+RPWG+gVmKGrsbjClvgyIO66X8/CadeERigbkE5bYZMN+Ijkogjl0zDibq4cNBBRyaKtq4uyU2OP/E0JDN9spk8kCJUik4igXiqOQ5aeGg/2mJw6HFpGI2GJlZNUnOxmIE5+qCbskmUY+aDsoYuSVOdSZty+jRoMic0GqX+FIcDZsNK6NddJCwKeWzzmnqDSWoEEU83Eg2AtC6TT64VoV46o/CHcCSVSohHnp6eRlsu14qe3KiMJjQawjHif3pQjQJz0MayRb5gZI0c4+PjyOVyqDcC2Th8H16/Ta71PtWRWnjGdWYuYZPN+d/5ejom6zRsDYE5WSymuJ+xhkwSN/OckQuUCVBrVHHPz76IycOH0NGTU2ZCFqchF3p07AhSqTSmi0WEHb341YuHECai8GlUoYN6qYyMH8GmRx9H9ykno1ZvCsadPjqGVCyBSEc3kt39mJieRFc6J2E350dQfnQbpg7uwve//h2EzTru/du9uOK1r8PR6QncvrcOh06YoT5o0gGiRqosogWSmB9DfmZaiiLi2QXT0s5D/Pr730JxYlgwIheYVJ6ETfK29DTJODKZnGDO6y46Hou70+Jxho9MYNExx6Ktd4W8jxehsWlOYB8EcaPgVIce3lfGyNfEshWiQ83wSWHaDTJHPWpxxdJ7EimYyLNgEyon7RqIZBNLTbIMviZul2KQa5JNX5wR3996e1KW3DSJZELWRCKIxfl+xBR0NFmVTcZrbRWZPKX2XEIKfmZNII+sI3MTfq5sRtJ5WiCiFyevL/cMvISR4rVXK1WJbGSICHEZcZRNUWKA70P7YiQL+axNDsT/p2Oi01ToJE8DTUm61Q64+RhVeB0SXcibMwm1ntxinHv/fBtm9mzQB+KGgpvqVb1o7jZ6En4gMXuhOIPnollsnimJFy0WZhFzPITlCp7Z+CQWrFmDRiqFTK4dCd+FFwDlaBxee6fEERr5nhd24YQ1x2N6/CgOP/AgfvH5G5klYveLu7Fu3YkoFKdxx3PjKCCJGm861B1eLpWQTKUQZXjkYhcLiPiK/4yvlV285cG78cSGv7aSPMIq9eQxhC4QiceQSmfF2/3bucdixWCncOileoDOnn5ku4+VzL0ZzoVFegk+aBoTF5SwhQ8nbCoHb3E1F12LOU1hSZSZUQyq9KMDhn2+h7AGBkpIBc9l8lTVPEoMWw2OUMSGbWUUlH4Tlmk2L+vB968bHrs9l20Vg/jsYtGYvJafRWNjUmjDvkITGrneBw1e4Y/doNxUSiXyORBmcZMLnGXy3LpH5bfnIg4T3IZc23wPzgSV/L6lRgWDCwSKGHilntxCwmq9LrkFr9NWOPk8uTnmqFg+E42UZJYkh5hv5Ew9/vTTG9Gceh6VBiuDIZLJlFxgJBIXg58Yn5QdyDcuV/Ko+z5+PVlANJlDpVjE9PikYOQtTzyFVSesw2QihnSmDYM9XZg4fARDx64AU93Ozm4MdPViw3334YR1a3Bo2w6MbX4Gf/nWLahXyvKACXM8P8Ctj2zGeKRPWBKijkqtibBexWOPP4FXnP9K8eBOuQpCdcWqmmmTRuzyGvjCpz5sqn+MSprQsOIZuo7g8lQ6I+Xt15/QhuMGO5HK5RDPtCGRzqGt7zgJgSTzaCSKYU0CZYyWRs6Fjws+VXgwn4MWVqMZyAO17ElZkrVQwj3DPr8iTGaF5gzgR0n51TSBMzDEbmCl1Qg39AHzuZRKNDZ+blMMQXFvFbEocW2+RSGSiyb0UV47RNJwzbyeXDar+Yrvo0iGw8gCfM8XrjoWVzimnpLMRkxYEK44jZfXbtkY3pcWvLRARIPmz3gz/Hy7PtwcvX19qJTLsja2YMcI5LmK+XlNgrsp7SiVkEqllIkivDHRlc+GtkoIyXXjhmpw/RSuCLlp+MYQD9z6dUyO7BGKiGFDsHgsiZ///DeIxtNoooGjM0VcedlFiDoV1Cp1/HG6gmpCNQ4zs7MCCXZvew5LFx2DA3uGkWzrxJKTViIMqugeXIJ6qg1138XRo+NoTOfRs2gBjmzfjsahw/jL125CqZgnokI8GkfokQIDyrVZ1Ko11JsBim4c246Use3AJFKdXeDte/TQzKqFH1ZP47sOujCLr3z2Y2i6xJOhPgipLjrwGP7iMTE+Gth7z10Ir1bAytUnIJ7KoQkfbf3Hi74Eji8P1H7RG1r4QY/IqNGoVw2u1o0ghRUmwVxdU9SREr/Rb9CTCzyhxKFhWZOaKcxoos979sQzkWLTSiNDvHi/kLkSkzm9Kgn3hAz8gZT0AwQNIzWQjcKcgkmghndeh+hPKFswLAd/xvemkSfiCdQbyucrTclyv7I/3OzcXJYB4c+FZaI8gbideYzrSXGL8g6BEyaZpdPkxrBBl5CCEaoVhE2ZnoZucxUbUYi7SaEqlalRk/fN+yBTZelFpXcN7g8ZYzUoIQxd3P3zr2L26B7ZDfzwjo52bH7iOTzwt0eQHRiCl4jiz49sxkBnAh/7tzeCHHu1cwi37TuIQ4eGZRFIW+XHJ9EWS+PQYztQrjRQCCtYdelZOPUV52Oi4aDpepgpzKIwO4Ml/UOIHTiM665+M3ojMRRKEygVp4GAFdcKwloTDTIkTXqnOkpNJoGAk+3G09MJlLw4QM8o+JSFIA3hRAtes4rvfeFjAo/kwRpjCx0XDqmumDJGXMx3nr0ImcY0Vp20Hsl0O/KlKgaWniLaEBq5GGJUIRvvUzlv4syKvEezzjBq9RaOJom+0bywUlutigFaeCLsDDU4hsvmU6DR22sl9adYXL/bQotuCCaxmty6Ljlz0oKe5DhzmJ33S8JOPSHZFQvmCGf4M+Jta8C8F763eFzjIWmsIkPwXBQLRYGI5XJJc4kmIxrzAVKNqh1h5FHoRQEdYVMdHmURvlKLtuLMzcH1YIKsBTI1SGJpSZR9HzXzd4Ff9XrLq9tCF3/Oz+YGsdDIVl4191BI6VRLM6FQV6xGBU387bafYOrAEwTkImBKJjKIxbP48Tduxv7hI1i6/FjMVAP0Lsri7PXHghihnszg5p3DyBfzqn6Dln0rhyZR3H8UJQlFAY5/7VlYfdY5GKvUkcnlcODQEZzXuwBXX3ARUhQklQsoF8ZQmhkXA282tdgh1J/haCUnCByUa1U0/QzKYQIvuEvwwJ23IZtKY3BoETJtnYjEIujp6UKpXMQPP/9RYVxELMXAxfdkmu34cKNxJJIxWdjLT+hEKpjFyuNXo3dgAOV8EYvWnk8EjrqUpl0xSov/hMvFXOEhEF5ZE0NiRhq8KvV81E1CxNczRFveV4yTdQpbjTWAVyt2et/qGdVr2aRVKUoqARUTs9DCpIyUoU1E1eE4gsktBULoIbkES8PG4kWHIgWpQJgXKXaR8TBQQa+D2FyFYvSchAx8FqVisbUmWh33RC1KLp92xShJYxYywOBrGjY9vOYnor6SaKXRSaUHCls0URaIyXWVnETXV4RfhC+Fkty3VnQZtUhjxlqJtOQT00cOipGHrg8vbCKoFrDhD99BucbiBrUFAXp7uhCPp4QpOTo8gsdvvRfLz1iNeHsKbtRFom8IX39qh4iP+FApa02nUth170b4TQ+lQlEYkQWvWIOTL7sUO4ZHsGjhAjjFOn7wT/+K0f370NXbjfHh/Sjnj6JamkbQrKiYyTwIhRgMvyHK1SaSmThqVRaxXJTCGJ5+fhh33HUf2rp74afa0Tc4hBWrVyOWyeF7n/kwfDQkobKbRsKnF0EQiUopnaG3PZjBey89Eel0Fzp7c6jWXfQtP0OKWTXjaWyY5wLTG9LALG1HaDCXdM5pLcSriKqPIiRH2RMRSHmYGB9HNOIJ69De3i6JnHhTUpzUdBAfF4tIk9oTOaqW0vkzGgg9t9WxSFk/qskWXyu41RiTCLDEcGMqFDPJpNWqyHWbjSNCMEIYY4D8XXpkugYr8uIGUxVgIBGCkcwyNPxcJq38DEY5emqrUGS0oYcXea3ZPDaHUgNWTZCNVsJ/0M0ETdRFdqzJt5VWcOtMTU2js7NTC3Bmbfl7hHX07M7onu1iRrwoxUwBNj90O8qTR4yGmnJKqtCogaiiMF3As394FMmeLPpPXoa2ZAqjmU7csvEZuI4Hh5lhxEc2ksDOuzfKgyrk86iHAfqPXYxFF56BbM8A6jEf53QvxPtfeyV2bH4GvZ1tGBsdRbk4hpjfRLmQVyBrviyHXK/xIWtiJXhMmABiTOBXd23EXU/sQGdbG2KpFPoXLcLCZatw+89+hAhqUgWloRMTagnYQxjx4EdjYjiO64sXScTieP/lJyIZVLH8ZRchGktqFDC4V6uWc3plKctQHEUPxGzfeCTxQgI0QymWWaMgzBDvSOciehaVI/C6JKkjrjXww6RLqr40Ai96byZ9tsKo3DQNd05y2qxryVuhjkbW+Yq+lm6dEIqQqNmQzWyxuVQxTZJtGRmFS7rRMumMGDXhFb/TY8/MzghEtLJg/j6N3KodPS+iCSRhnhFPEZIJR16viXcXo3ZVHiDwjddu1oXUrBadrNhNr4fJaFubcvqkcefLlsVudm59NFTNLhMFJe+dsIqtG+5AqTjbChuyIwDk8yWMPPUCRvYO48TLz0EmlcTNm3dhvBEiEY1jcnwcR/eOws1XUanXZTEY0shxO4kojrvyQiS6erFgyWJ8+43XIhONYPTgHhw5tB/dne04MrILtUoeHlTPYDXDEsrkIc6VijWMOggNLVepBXj3J24So01kMoimk8jk2jB6YC+a1RpcE/rkxnk3jocg4gpUkxKzo4tLz/O+y89EV6yE4069GI4srDI2sjdEMKVQyhZCLBdeKBbFAFk5tOIhvrdyJEwOlRmx5W6tCIYC6SwOFoO00lNjVEyMtbGATkcTRy3uNAUjWxotnc4IhGHSzeu1ZXaru1EuWo3efuezZaJpjZwJqoUKtopID2wNj0alRSojlWWJPhY3sEXAvBimrURaBojCX43IobApIrAyEUYrnQp3bEJpM1FJ7I1iU/MNfS2vjbDJ4nDaQ62ikGX++zhPPHhnyA+TbNgI9knSJtwKNj14J5p1dmXE5JeHDxxEpqMd1cPT2P3wNhxz3lqsfNlpuPbGn6FWLmNwaBDZRBo7t74ArwHMFvOCp1gwoIFSFPWK696BYuCgf/FifOeN70FK8GoRW57aAJ+JQmUSzVpFoJJNKMRDUVcjnSMKHSTxkzKvejhJQup1XPPBr6HuJZDIZJHM5aTSx6othUfUrggyNMwCjbphCj00bDFy4Z2jWNyXxdWnLsBJL78UsTg9udHFmNKyJI8tfbfClFgkJkUOeip6VqHdpMztSdFCjZghWZssNM9oyuul6kkNtzFAMlRixBKilSO3AitbqqdhSEQxmnZVASqfzzyC28ry2No80ZCE0aoU+T2TyRhGghFIK4TWELm+GlmIqWnkqkch/s+k0wJvGKn5vlbPot7WFcmANkF44o3ZnKLadc0/ZC2I0aX2DmFxCHvkOYgkl7KEujBE8jqjgdHaqtULqY6eeN5KcPm/lt6kClYi9H13/iKUECt8pmbhvFHuVLIUYwe3ozA5ItoLUnRMIEuTBWz7y0acf+3bUO8bxCe+c7NQcpV8HqWZItoSGQzvPyCGQfzFLyl7R6JIn3E8Fq44Dr0LFuKNp5yNK04+R25iz/NPol6aRmlmDIHIBLRcTNzLm+DiJVJp6fBhAkLDIy9fKRVQq5f1QYfArn1H8clv/FKS5ngmLQkQF3J6ZkbuwWUxxXadeBE0hR30JeFih454ANdBW64NH7rkeKxYfy78mFJgkrSZqhw9qG2xUoaiJqFSlXdsydJqJL2OLevbhMp6RIZdal3YyaMGRSPX9jhGGuWONS8hRrdiJkIAGhWpTVtt5PraZE2xrfLdhEn8srDFJpF209Arz/eSTC553SwsqVYpLvdNHp38O++LsKSzo9MUp5QqbZXSLZ4HowOLhKQ/tWJOKbfcj6ES6alJUzLy2CjGPMzCPysi45rzGdImpc2OG5mb0W4V0sXmc0S3ZCKC0JlctZ3bHg95AbVK0YS/htHfB1gAACAASURBVOgsiCtJ24UNarhrqFUL8pqgVkc0Esem2/6KWszDeP8C/P7u+xBLxqXi5zYdHB4ZhtsM8da3vBU//9nPpIjDCilD3tJXnYmuY5ait6cf6UaAG993PRrNEPt2P4vy9AjCeh6ewwSiKp6NOFXwYxiivaMf9dAVCDJ1dASF/ASaDdVIi0d0AhRmqvhnQpZ4HG1dnZJP0JNMTk0JJhddiwmZxOAi8jKMCRtGbBmbnuo/L1iGdWdfAi8ab8lOBbZJ8qj0HxdfmiLEk2sxxvZPKvVF7t6VriH+2+pX9KEqYyMRwfRzipqP98NoRcdAeo00mckJzHM1lUcVUNHradKpTRgqeqpI0sqNbZNh8fAiltL+TAsnbDOIYFqyOAgxPTUtXtDCJL4nWQyphrLrptHEbD4vkco2YLCDSKS7iYT2udbrovHnLqV3ZRShMxF7UDykEJkdSGywkA3iipKSr52rDqsaUqqjJoJzHSxVyvukQ+DCy/WbnIl5jRj56PCekFmr9hTWtSm3yYpUDU3KOWtVhMSRgUn0RCccYOr5nbjvu9/H9v4BzMDHrp3bVcQk7xEIU/Cef3kPvvylLwqOboZN9Pf34ep//Wf88eknsHbtCfj4WYswtPZqEe44tQa2b7oHvUMLMXZon6j34rEIZqcnRRsSNhz0LFwqfZjxaATjh/fJg+R1Mj+1cgN65rf955cRSeWEpvSj7CBJYnpySgsIgus1AeXGcynwilB1x3xEPbnnU3OdxAcuXYt1LzsPrqv9oEodEkaFEmHUAELBz7LJTNMA/07GwxZwpEWtyhY2peeU361J6Z5eW8ripkhFD8XfZ/gW9sFIdIUWo25dvBYrkiUN3JQGp1LifWtNasi52agfkecrUVAiByNtqWgMW1sIZwtaPbSUqGhnDK8v7JOpMgkcMH2rMzMziDF/MQpF4aFdRzaaVE9NBbbVl2t08VbzYnM/jXKaQLLgRQimzkGLdXyddiFpImnb/ezm4WayG5+QqCPXhsnJSXHMfB9uUEsrOrd87/PhiuWrsHj5CvgR4l2uqxo6F5jkfLVcFJ2xlpy1vzDRbOCv138aOyamcPfMLOpkng1Gpq6bF3/FpZfhn695B5Ys6UexmBf9c9CsosHm1XQS5eFHkBg6H/0L1sL3Ytj65L2iiKN2Jaiz4XlaKnZsDqDAKp7KgvoFeVjcoZ7iNTo5GnmVzcy1Mn5/91P43UNbkMqwmToqRp4nXGFSzW4UY+QSYokzo2rA7FyRBCtsAH4Sn3nbuThuHYtBUYFIlge2zIh4dBY+1J7kYQisMe1g6qzUOahAi9hIPZBW5jQaUE5KTy6VSMMoMBkVrEuYaJJF8UqmQdeWv+k9WXsNamWEFDo1qlJgkxYwQhhRC5bR3d2DYrmM0NOOGjYzV/MF3XSegzrXPAgQjyUlCWUiSeO13TdSI3Bd0QwxAtiqp62Q1hg52AdqS/Chg3x+FqlkyjBMmh/wD700P4tTF/idPDqdmmWjuBZMxOWz7ZQEs8bKtmguMh+GlQoFITmmZyaljY4wkLSiUKU//vbHQlbFKH+sNX3k2vtxzMo16B0YRJ3ertYQloUhk4kdvSd/kX82XP8ZHNq3F9siAZ6amkVIL+8AV732Mnz2M59Eb083SoUJFGYOq4GzXFwsosCmjEYD/akGxifLWHnmu2TRGpUCJseGEfVdTB3dDycoyc5WdZztylbBk0hF2RgRJVZVw8nni/L+ew+N4Maf3IN84CKeSCLTlkM5X2gtor1+el5JuunJ6cFNyTvwKNN18Ym3vBonrluD0IsiFk1pAsSQbQo6opswLVzCS3u+wBfB1YYzZ+LLh2fFT7aYYUc0qM6lJp9vy+d0RYRpklCTmyaUMU0HSptq/sSoKyX+RhXbHrkTs1OzUvxi6B4cGpI1YaO20KUm4VavTsqY2h6lXh1i72RaDNCLELJ5iEbjkiDXeLMm6fR9dQZkcAg/KtSec/25cR0f9PK8d94TGqE0wDCXiKWYHEakc0rqcdIQ7cOXUR/MB6mkZvKq+Yh6fXLypnrKSBGLS7RSYdicvEJyDcoHqlWxoXRGu4FoN2zMECP/4x9uD/Oz02hUZlCvsm2pgsULFmFk+CCicR+xRAK53sVYumwFquUGSmWdn1GrNbHpR7dgxz13wkMEDyVdTER8xD0fs6NHsPfFXSKWyU9PSkGCN0J98qGRAzi49zkJxyz3h6Uizn7NNSJvrZcLGD98EJXSLILaDBpVNiDojRK/ajOt4mFhSITWpJKP5XKGO+24OTA8jC27DuKXdz6JWCKFJAX2putdeHITKhXz8iGpdxNPZuZ7BK6Db33on7Cgt0eM3GHskHYYfRA0NP4ucaJABdNXqS1c2p/I99POHKW8+NDyhbxcu5bFrZTUkcSO18AqI3+u8EfqsvK7hDFMEun1eI18qIy00pjgudjwx5+IjojRQcaH+JTdRqk4n6vQit5GMbeNahoZSGkqO+UEZlIAmOx5EgllUxPOGt2M42kOFPXYS6nRibp+YTgCU5mFJtHsisp1dErC6viEOS4a7DCTqmQdU1OTqNcDdPf2CATj5AheO2W1VN7xeinaFVpTorCOJLGQk59BByzfpYlamRnr+MROtmx5NszPzqJcKaNUKgisKJcLshRBrSTip2iUs0U8HDx0BP/7NY54oDcIsSQaxwXt3TjCUBlN44pv3IBlC5egrS2NicMHMTM7jaR0TodYcdJpmC4UpBF5ZnwUe3fvEPzoeyGGlq5HZ1e/4MTDxONOgFp5CsX8mGGXTVnf4DDeLA2no71DjYb9foampJGV6008+dQz+NvjO7B9eAYZNkX4BiIY1kMMyIRW14kg15YT2EBKrVxlEuPhhv94K5YPdcONZoSl0cZfGrkWMOomsSFDoO8XSAFFk031vjac8/8tnWe7ZWx4JjSx0UWkrMbrcuPwvSw9pwU7V0ZESAVS+GyKzuq4/3c/Ql/fANraVElov1QIZYpSlusX/ZYWouxrtfpIA7fUrNYAGF2sLJfRUwyoqYWrptmASq+aAk1zrsGDHlf4e3MxlnyQWSh2s/nKGnHmj4jXKFk23rql44lkVPsS0aFKMl9FJMIhqkSWpqn56PhR4frJAslG4MQdTibIFyqhhJ4qu4BKgsfYS8hycak4g6BWQ7FAiqeJeo2l9gD5UhG3/ea3+O3Pf4FfvfMaXPuNz+Kzb7sWfeuOxcpzT8K69evxu9/dgb179+LIyDg2vbAbTjSNYwb6cXhiAkMDfXjVRRcKG9K/eAmWrzoVPb39clHkzMdH9gNBGa5TxczUhIxZ4LAcFUZpUYiUHXEmZaT0nDrERznSaDSBHTt34cV9o/jhnx5DKpFmjGt5Az4+60WZ7bNw3NPbg5npGTHy6eIMfMfH+99+OdYt7kGqrZugQaZvMYnu6OhQ+GGSOkZRGiNzGXas8BpswmRL+ZYJ4Hfeh/054RWTPbILTNxsdc82NZN3p3H7TIw9VhDnCbA4NEm01A7GdjwOis6YA9iEzBo3X6NVSWUs2N5o4Yt4PBqckQ3b4ozVlNt6AN+D1ylN2oSlBjrw9+XvZmPyu+XrVXY+t8ksbLKFK3t9Vs8uZACvzo6SsLNnyMaQGTO5nq1PKCOlUckyRGT+amQFGX2svnZ0fFIqnsRMoltmqKxWxcgpgqqVSiiX8lKenRg7jB98/9uaDNYp6HdxZhBBKdbE3tFRHBtrQ+7EJSg4dRw8eAD5QolbHnV40v2OwENFksgG+od6cc6pp2HiyBG84wMfB1JtSGTapPikRk4Z7wya/CzpIWXCOxfGfT8uCQaNq0yMz9BtPMfs1DSOTsxgYvwovnPbo5itNGWQkJbGzT0SKpCpoLjHVbjCRed7lmpl0dpccvoqXHr2WsQzOaRTHaLtilD+a4pJHKsnfLVr5o7M06doNVI1GDJajRGmUm7RdoRXjEbKW6tH5TXIYCA2ObOhIcFuHuOFzZgHFllEBCdJqkIaqQO8uImCY7juSw1Q9D5GyyJsC/MG14rerItVdWYrAsigIUYl9smqWEokvjFdIxq5DkIyTHVLvmAMXHRBc2MtBBcbz203w3zNjI12ttJpx0nMbRwTC0JT+DMOTQtEqmFn1VsSczbkciMyTwgIXxw4W3e8IFcq8/AQoqurC6l4whRXlCrj06Xx/cc1b0G9RqMvm2lNDhY3XCzwgc2Og4FSGe2JOMZidZR5QYbiUuPUMr0MLJK2JB/v+a+PSTfPopUn4OH7HsRV//wvaFY4dKaEI8MvgsWvarmAeqOkCZ0pp3PRct2LJDmamRyTa+OAIXoyGlUhX5QJXXk2cZSq+N7P70NIHQeXg91zpil67qHPSRokMdNWdKw9pg/vOG8V2jsHkMy1IRZTbC8N0y7lo6Z4JBJR5ev5+1KVFY04GxrIYTdkGpnFkvah8ndkvATbDs3EK96blvVVE8IiXQufG3hliyE2SWM2N7Zzo4yrYy7B6xcow/s1lKnAoab2jCo7JE/nJdBGPCypQnOttBvbzib/ZzCyjMKY92Wjoj5vM92K/a2mj3S+TFh8u3EOUhgyjBGvTbC9TZLFc+sULB1zqF3L1hHb39M2pbmvVl8Y6wFGc+787d57Q940s2qrc8hk2jT7Nbzu+MQUvnzDp1CZOIjp2Vk0jCJMOksCF2chgqc9dss1sQYRFKNNHHH4gLRzY+HgQEt5x8yaN0fp6kdu/CWS7R2YnpzAc48/jPNfexmCug5rHBvZg2TMwczUUQQBp0pVVXVKI4CDRctOwsxMHqiXUS5MolaaRd0kgMViWZtsoxHs33cAz+8ZxW/v3ypzVgg7RAogE9jUW7GiZ0VE8t3l7MMQHZEYPvGuc5HOZZGIJ+H5CWkccdmZ77Kwoh6mSrlBPKFqwXTaKO4UM4p6rt6QNWtV7OyIMzPFKpbQ9jHruaQlzoxoq8n4jrn+UkkY7YOlRoSsV2ka+dHnJfEmtNHmCO3lpIeWohRHyLmMOrqJ1QsblmaeR7Zj6ZiDWMGYzRekei1tstbIVR1oPbrCFDMUSfaXKcbME9opRNFrksquqYhbqNIyV3HPFm9o4ciqFc1CvfTfZrPMZSOAZ0fu/fInPwy5cFbfLBXCWFIWSytXESnH3/Cx/xIV4sTUhPKvbH9jQSNo4LRmCiPRBoqZODqqAZYELo56dUw5HErZwOIBTSot3OB3trC99aOfR669CyOHJ/C1z3wUN/3fG9E1uBz1RgWlwiSC0rjAImnXcnQx+Sfd1o9YWz/CRhFjI/tQo5BMRlJYDbZqvGWzjB3F7t178LVfPIpYykeD5TaDHxUqaHHFltq1zUrb/vgen3/r2egbHBSDTiUzcLyEts2RYvPjKJbZXGKYFCZRMpGKzIEmnZYF4hg7fgaLL5ZSrJoEVUVXOtqB6yRj8ESjQ2WelqbtlC0bHUUgZgaHBpVpVMYPmsYKO5jUMCjmGvheMr6BRICpNortGbwr3th4UpuUc+Py91oskJ1CaycfsLvcYHBtmuDlz/XZWlhnG7VFxc9qJJkwmfGiPZz2dSqdVwho79NuIIEdVl8uDIs2Ss9PslXVYoV0XHsWqlw43/jSZ0IusIrcPZVwMhWhgs12dEQiuOW7NwqmzBcKEn45UmKoq1eonij5yUQKhwszyGVS6J4qIhfxcSgooug2sGywX9kaU5zg75frIZILjsHlb/pnPPL4Y/jtb3+D173+SnzwuuuU3QkrKE4Ow3NYRCiZkRQ0dA9Di46jmAPD+3fCCarSkcNCSMPw9+rttDhTKBQxOnIYP7j9ARyYrGry2WrEmBNraYVNsTnDJLEoX/e/7z4fqVxWu9E99rkmEQgs4MNUDQ1CLeSUq3VwHgihCaGUVCjNgwgNNWehitCwZtosI4nmCqrbEBWfmaHC5JbJKGEjHyphDR2SLcnz/SOoYmLfc+K2+Qz1S5sLrAHR47YkCZKPaPue/X/rQOzG53del4V2kvNwMq/ZXCrtJZVrGhvmGXnrnk3uMrfZ1YvTxHWDqganFZn+zmhb18YIQYxtfk9ZLDNzUraJQV9GQ6PiNwHo+v6f+tC/hZFITMrf1PuqR6dKLoKoT6+kA2Fuu/U34lGnp6fEWxFvDsXSMlio0AjxwqG96OvqRm8uC2dmFse4MTTdAON+GZmEJomSwJhueY54nqJKrGsRjl93Im67+2/oO/Y4fOFjH0RHgr1FARqVadRLM0alp80CXKJFS1dgZGQE1XJe8LgUTghjmnMzAAUH1+uYmZnGxMQURo6M42d3bMBY2ex+aaCQxyELwerYTCGvmbrnIZ1MoVau4Po3n4KFCxag3tTJBXxIsVgC1VoTqWw7IjHmL9oeR6GXcM5kQoyeIpXKGL5bu4TooUM3IkUQJuDkvjkFi9/tOAjeC2ekC++rsnNRXjKi0ui0AKZzvpnUhrUZTB14QSTB/Oy5B2yaXVvKG9W2a5V4LmnUopYmk3YTGvWTYWPU2wpGZtmdHLo0Xih3LbIAOzzU4AWBgvMMeC5J1TY9fp6Kz7TeMX+zGX/cQiu2OERPrlIDK81SVafdVMoczb1Ghi+Jkf/XO0J21/C1nssOGWJP/ptlbhfJBD0XMDo6gq1bt0oVixizGgRIk6TMF+Bnsjhh5XI8sWMHMp05xJwAiUoNnWUg71UxHRYxMDCoRl5XT0rmplStS4GhIx3DmhNPxGTDwZLV63HhhReBqLJWmkKtOCkcKg8DIAygsVGNqPMPy6hVi5JQaXhj36LO5eDNT05OiYExCR0fn8JzB6Zw29+eMo7ONjSooUuDgVUC+j4yyRTqlSq+et1rkEkmUTP8utTrmg5yuQ7p4KeRlys1ZPlvR3X5LNhk0uyKrwl+588IO2ic9UYTX/zmd7B794tIp5MyjH7VipU45ZRT0J5NS3f9nPA/lM3CjSWjiEmtGdZCijHRqOQBqM+KkSeSadmgekcvNTI1DDUOS7da49C5iyrptQUXrpvNIcQpStKnvZZi5CZK2KjIHMLCHBNKXvJtPuzg/en7mJrAvKZkC19Ei289uKmAWmjfgjdyYfNRuGn+sZ3dUgoDnP+5/q3hli3PY/XxK2Vsc7nMEcAM2REp91KERONimN/w4Aa5uanpaVl4GdhDgVSziVMjGRx1Q5TaE/jJj3+G4UMH8MsvfwP5F17EQXdGKlrc+Q0zDJ+hulxvoNKooj2ZEFXiGWefju7BQXT2H4Nc/0LUggYaxWmksxnkJybks6mx4OxCGRFRLYmRy8MX6amx3yCQErPO6GPUqePg/mH8+b7H8fD2IzpdaR5XTk8pc0LMCGEn6qOXWo+ZWXzyXeegsy0LptBipPWqVALJIlAjzQRUu9HJ2SpfK5rwgFKJJOqqhQJxlwz8cVzcdMsvUSgqG8N+SOG25ZrZvM3uFkcMvn9gAL29vVizejX6ujslvNt8SDyoGejTYOP32H4wIgsfb9rILCMx5/3sVF71nHN4lgUlbeSgwxBdTRjIBhSoaIxcyRrtw+SG4OtaXlRwi67/fJzMf9vZi9Y4CTvmune0AjvnjS34sEaujIrSkHNfLRbGFKTsZ3Lt7VcLk3/m/W8IJRkxeYOo4coNvHjvMxg6eRXQmZbyLUc38EFveupp8fozhaKoxygeygYhTnaSqEVcNNetwGdu+KxSkM0A/33FW2XMw3QHJZYqVJKEqsKG5CbK1Rp6OtrQnk1i4aJFWHPiOnT09KJvxTopESdTaUxNjsIjI0KS3+xSGRncYGQgJuf8Pl9mgOv8vooYuS24cEEYgcZn89i6fS9+dNu9YmwI6PWpRedm1ulP9IRu1JNpYeViBV973+uAZlkqpnyfSrUuhkd4IYJ8em+Pwz+B8ZkpDA4slA1AGS+5fPuASEmya6hUqeHTX/6uSEplYrDo7NkSpjw5P58elGo6GgKPVWGTAusW3KyEfYmIK6X7VSuPw9CCITSnDiDmNVAvlxDPKSxk00mTsNPACWtE1gOrt59jRsSQZWiSLbZVTZI8N6VLJMqmiWG+MVv2RURcFq60GByJHWJ3/D8xTsusyOaZ88Rz+YNOKRPoZAaMWgsXTD/vkAKptOpRFLq5jI23NhTzs+vfc0lIw04ldW6KKOLYzVEKsO/JbVh2zilo+g5q1FKARpfFczueR7mmb0qcfnypiZjM6wjxybtub1FUXLRStYQvXPwGFOPAwLoV6OzpxrNbt2JyfEImYpUqVXRk0kjEXCxavBj9C4bQ1dOFtoGFGFy2VsNrsyz8ue8SoKphsGiik5s4uozXojJhFZGpWMcq9RQbAqViGaOHDuHhrfvxmz8/DsdpYGlHFL1dbVJIKtUqKNcD5GeqcDhCrRHi09e+FomESogp+q/UzAD4ZEK00pKQeap0rLDJOJaEH4mhGbKjPCHKC4EHkaiZFuvivR/6tNBwemqGftlpVax0ah8kJQ/awCFet8kudEYMOgkdYE8cTBjEDcHpZMlYiN7OHIb6e3DMon70dLabMXOahDLP0T5RNSybn8336hb6We/dMkIanRyYofSrXvSc5269p0lELcuhXloFfTRyPjfamcAjGZz0UrhhP1eeu8H1kg/Mg0cW08smMPUY6TDivRnGZ34y67z/Xa8K6Sk4L4OehPhVZasVpGtA9UgBkWW9SObiiPsxmT8ondqROCYnpjA7Po0FR6pYff7LsW3jRnz+9l+h5DIhcVAv1/COd74FSxwfqfEi3OMGsXjdKhwaHsaObc/KzdaqZWEy2KQQxKI4+eT1GOrvl/L6gpUnCHVGL0yFIn/GncrEmN66o71LvCZxGRs6+F4inqIXlO8qPCJMouaB3pd89f59e3H/fRtxwQkVxLwmIg7ZDRUC8cuKZwXfkrGIUdvSi0ymB/DimC37qDay8KOutLyxhY6RKZ3OylzF6Zk8oomcSJfbOruQzKSou1NjDRq4/C3vNpN2lUmZ/yXeULCxqeC1YrT2tspcFwqAZBbhHPXJ95Yo3NAzgur1ssAj9npmEj4iThM9nZ1YeewyrDimRwzUp6rE8M8CQSjvlZmWZFaY5JI9UW5cGZJ55XtZ9rmk7yU38Xcj8Sxu53ep1MqokbkNIhvO4ujWepgk2bYqzqvIymvnYRet+hqYxAgtLFMTXmB6lq+58syQxlApcVF0cqnII3mmjhNB9cAkJqZnsPz049Hk7EBOkpW+PIbZOM6/+Er85D8/iYGTVyFWDrD6opfjuLPOwZZNT+Hm734dkZCjlhvoLoZI1YBV77wMiVgMO3fsEK0G9RAi8eROFUOj12GhhQ9xrvwsWEvW28eFl18mCjVSd+k0u7QDVMi0NHSCFaUA4slFUzE3aYkecnZmFmG1iNHnfwevUoLLzhbDKpCu1HtT6k8wqqHk+PmRmIdsLoNYMofh4QY6Fp+BStWMh6s7SHT2oW9wscx9UaGV6jBmJo9iYmQvhvftwcOPP4HfbdiG9lzHS65tnmM0rMQctuT/aQFFjVyvjUavXUS2QCSbiMYr2ncWuShBLUtxixp+9g42iOtpZHydo2cvtWfjWLZwEIO9vejuSCAt49+0aGZtTvxxaI6NkQviW1huXDkbu2YtTD5v/9rxeXwGdEYvwddmyGiLCxfu3MxQNxNq7S9YTf78TSUb0OpnFCCKI6DsRN7z2jecHcYiroxkI0ZklZBhjRSPaJWbAZ7f8CyimRiOPXWleE4514VvxHN3pn2MbNqMzpevRrrhYWTrLrziXZdhx+ancXR0XPoBKculbLd4tIr1F7wchdkJuRARHolEVrlSGryUbdkW1ipMqJHSYMnbytyNMMRlV1+FUqWOZCqn8/44oL5eRSPQ0RMM44QtMpGWYb/ehBNnqdfFCxtuRr04I58lQ3aMDNZxlZF46ZeWm3llNKZoIo7O/l6MT03Cz12ExWtPQrZ9UJkAP42wXkG1MIPJiVFMHhlGfmpMDxaolKWx+4GNL+Dhp3fLsCBSq5F4SqhbwhfO/pO+2IgHlymIafwVIzZzhhQmaGVTJmcZ2pTXaNkN9Yo6uEcmWcncc0eauhk92aCgTRva7S9cjNGicANwkyR9HdKT8mtYfswQFi9ego5sStiwCPX2QseZpmd+linyBMKLsc1Q5bACwyjjZRWXzfLsxZRJXqp2ZLIvm4Kctpnga3x8qzLKJ2JtRMbxmW79+SyLjTLca3L/omhUR+Fc/+aLwnRPVhIobTHS4fUM75QsilDIj+DuH/0Ba84+BR3L+hBhb6TvoK2tHw9+++dYun412lctQdxxcf8Pfo3L3vsWOddz27NbhOFgta9ed3DWxa/GIxs2SIHHHqFH7leYETluT6uixIr8mXoEc7qD6c0kXhHtt+/gkte9XjpdVOralIkBjWZFklsWUKQpl8mqtKhx8itQG92E3VvuF16dRsANIJVuuYZ5YbNl6cofkyLTHkJPZpr3DvZj1lmBJSe9EbV6HuWZcRQnD6OYn0WpQGanjHKjLhpvaeSt1jA+M4n7H38ez+4mw8MJXh6GejvwqnNOk8/etXcUR6emMT41rUcyUnBlKoJ00a0NaEK7YlKdS2i1KVaewMTaiqIs/WcTNlM61A1lyB/B/8Iz25MkdPJWXRSV5kAvRnLOpvGaiHk+errbsWTRADpzGbRl4ojxADFedeiJwlQMzEoBjIpR2S7tB5AN2IIn5sCcefCtxbP/XbRSPzSfHdIEVgYOGRxvkYFcw7+fsTo8640XS/JkO81BIxZ2xOgpggY6Gjn88Mab0HXcQhwdPYJTz305Xv7yc/Hjj3waZ1z7JpE8VpsVjNz1KM5806uw+ZknkcvkRBLLpolE36BIb0XgxBHHrnpYjteVrnc5F8aEZXYBzRPIW3tj1Y+DhHjzhFNnnHseOgcXtCp5dTmiRItDWl3V1jmJEk6IbNzHI7//MsrluuBPOQNTkjtV9dEztrBhiwrT6pptCGbuy4m46fY2jE1MoHvV1SjPcuoVD7uiTkX7KaiBrQAAIABJREFUERukP+s11AOV//Jns4VZ3PXgFrx4aEbW96uf+zCGt280Y9HY7c8xbxEk0hm0dQ4Iri8EUYwcOoRHn96CXbt26XMx0IBxSQ4CsHJW02QsntvROS0KddSYjUykpdybf6925o6teGpRiRMQODOd9iDtF8LahHRIMnqOVCPHSegJcZ5D448gl/KRjYZYtGghhkgJp1T2oNMF5kVLwUB6jXbyQEujYrUopgilOYHB9EZ81qIR5b4tl6/WIq8XyOvCue7UNeGF//Y2GQxUlmqWagRmpqaxZ8fz2Pz0M5iamJaxCQxZQ8uXIRKPIhZP4Omf/Q5tPZ046a1XoFmYwdP334+lqU6UE1GM1fM4OjaKoYULsHBwIeK5dmzetEkWxtJI9DSJeFQLGDREc6HWe9uwxe/2pDCryGMHDYcCveHtb2dpQoyUencmpGy8ViqRXLSKkOhjDmy6A2MHtrfUbELjmWNXJKoKrccHOW+h+FBlUKjVWOjm5IPn5zdyZ6Jc1+4a2VhmGBCLXvw3e1J5DeVSDVP5Eu5/9GnsPVzAV/77Ohza9Rz8oCZFKDZhCANiVIwJJrG5LqSz7Uik28DKaYy8vB8VCPjhj/03Ro5OyTlJjG7zcbDMRW/9TNkN1aWop5PZL1QUtiqICnWEobC6HuPirYCKz8pGApscM7lracFF8MYR1aRxzTx2M1udKa50KrlM8gN0ZdNYsngAPd05ZBJRpGMcg8JmFCo8Ca9ohXYrc/PodQnDIn9T7CaV0Fb/qxWDab5i10PymF/8+7Uhvd1IUMPTW7bi6NQU4skELr7kNdLQ0NHZgdDiVsE6Gm46vShu/j8fxWvefy0aHW0yCmB2YgruwQnc+ptf4bhXvQK9/X0idoq6Dva+sB21fBmNUJsAeNPMAXhz9uFquFO6z05MpXFLWDaiMGvk9GCpVBar15+E5WvWaNGnxqm3ZUlC9PWKO/lgB3MN/Pnn30C5UFJo4pOqY4gOZSoAr587QR6gyXL0c3UcgoRVKYZo8kVjbOfJG+ExKDs8kUOZB+YOxJyMbPxZtc4T2yooVmo4MjGFJzY9j/e9++0Y3/ucGUKkbXUy99Ak18w9Mm3tiMbS8iwy2U7kOnpkYFKW804cB8Ojo3j7v/xHS0PT8thiELagYmOgTnid+zIGYdZ2Pra14wJl4tnfleXnb37rRcUpGApUxgyaxgbmF8KqmCNolEvXmeMcL8L1JESW06zDAPGIh3TcRyYTFxr02CWLpHYS1rWhWRxVa8CQOS9Vjs6xVKZiejsY1UYpuYc3nbw6PGHRYnRwVFoqjcRgHyKLF8HNZuRMzIhwwIp59ahvF1HXw70//CkOb96Oa77/VQmjI4dHJLEZyHXh9q98C6/893eAMlF+rTpuBX598w/Ew4pHYebP5EqMXauN1nAUblmds1WkKSakndmBjrwectP0qG9829tQpYyUYxcqZTQpfJKxcqywcpPVse3+H+PwoQOSwIknliRW1WyxKDecOBEtbduKxjxjEZjFziBT0ubiUXu/+0gFTsd60+ZF3TxnxlCXocPgWUd4cfgw/vbo08Kdf+ajH8HI9o2SqBEO8gGKxFlOOrZMiUYm8vJ+PI1EModcZx86+vrR3tUPL+LItNrXvf5qjM6yTjBPlWqbB+yhUPN4cessrPFa49Y+0jn1n2L5udOr5+2Ol/yVQqu/h3fy3uIE5gRUunnnvKvl5WVzmBzA6t6NVk0ku1HOb3eaYleu08BgbxZLFy9Bd0cWybgeZ+66zAFM6x73sjlTR3MsQ8NuuPtWTe+awPTBQ3jxwceQ4vnrg71YeMbL4La1IzTejAZKnjmYKODWT9yA5a94GZae/3Lp7pYgwgE0rodHvvdTnPauN2CmWpbkpVyYxeZHHhHj476Xs+09NahYVI1dMbEZ72uW0hIdFo/RG2i3DR+AdsdTunrKmWeib/EiaTSQGeY0dDPHhOzD0Rfuw55nHkWpStaGcIPJExee/Dm75NWr88GKhzLHlEiGbkQ/8nfpzjHdJjTy7m7sGZlBvf1UHZ0gVGZVMOpssYgt23Zi54ujqBI7A7juX/4J+f3bEeFMd86acfSQKCvztUyI0HueFrvi6SxSmXYksz3oGRhCtr0bqWxSZrH/1//5IB7bvuclhqdrpT/SZgUD+oyO2+JVTdzm/6rZYEJMzPVszn9FK/E1P7QR7//j+oXV0Ejwkigxr1Kp82fEo7W8tH29RkTlyeU1xPGGHpUpaNKNxT+Muk3kMkn0dUSwZuUy9Ob0sF29VlM5feLhu2R0M6tndpxu1HHxzJ/ugz82juxAL/zONjT72xHlyQO1BqLDY7jrB7fg9V/8OOT4Uhlsr4MoaYS777wfjXQMi09bL0zNhr/chbEjY7I0vqcTYVl80iYNPWeeVSxSU1wUncc393CEum6dOkZIUtPQhVDmevD6r3z7m4UP5u9T40FDY2GkMvoMnuTw0oI5a95RcRG9A3e60IIxUom22DJXFLIeT9aHoVeoL5PIer5Ah8NTBZRiJ6JU4UnTFWzfeQjPPLtLxFqyzFKJ83D+6evQn/ZlpqQ9hSIZV8ms0IeG3eDa6EnEqsdJppJIZdqQ7ViArv6FyHR2SoGMwrlPfuLD+OOGzS/hzy1G1tX7xzJWJv0C71gSDzlrhj2kVHIylBFTExETftGTEoIAToMRzjiBf6BPsUyOsFDzNpZcRQvSmKv6u+jCn86HF2L684Yb8VrVaemze8nGI5kt0DRENurjPa8/Q9bPvqc8w81P3BeKWo5Ym4ODSHdR2lksIeICUwdGcPTp7UhwPNtQP9y+HvzhK99CuqcNr/rgvxsFoMIJJhyCQ188iPv/+Becc82bsXjhAvzou99riaXY/CAaDXPQE+fH6AxAHnCqD0bIr9ZBpzYb153JaEF60P6d05xYLV22+jiccOJJ8vlsyqYUNizsxcN/+QUq03mBD9IZY96Xm4yOzvVZfqf4SotNEubmlastI8A9Rx2Inu7Aa46go6cL44Uq7tsexZNbX0C1aqAO2RiT4Qeuj6HOLM5ddxyK+SmJhIR8rPJyLrk2bDDE22m9Kq21JzWwVpFIZdHWsQB9i5Yh1dEmBp6MJ3DDDZ/A7+975v/j9ueSrjnO30ZJvUnFrw7qaPDEOvCI9iZWLhlAd287Nj61DcWqi8BLwmViLN0+9Rast9LXf+TlpR3CGLH14q0I8HeKQfv7klDayuY8VsX+3tz9zLFfrdeb8zuZCx23sAuXnHGcOE2dvqVjoJ0H7/mdeHKZD2KOCRFIQk7U0T5DHpkTj/jYeuc9GHDj+NOdt+PVb34bEuuOlxKtHg7K2Rgc+BMgWqvj9//zbbzm49fhT3+8A41iqTVxiZ5cEk6ZI+jCj+qUJqnSmZkadi1kqq0MbdfwIx5QZnvoNFsaNPn8zrZ21MImrnr72ySS5DkEtDCBZ++9BYePjiFoROE01ZOrkXN6LRMZLUCxOiae3DNH8olUV+mqeU+2dQaoRpsIegd7MZYv44af7ESACByPgi3TYWOKMSuXL8WJCzowdnRKWaRGtdVWyFxA8gNfW9asl9Lh+zrejX9P59oRiXehf9FS5Hp6VKQVi+OGz30cd9y/uaXrmIMic1HQcujzjZyeXD6j6SH0injw9o+jPLMZPjifHAgjKgmOZ9djfCaCq6/5kFRMbbPwPzJy+9nSbjfPk1sDls//OyOfvwnEkI3EQOog8/TocxJeo4FpJaA820BP36CzuvLcEzGY1XkvMriWJ2+wQv/Avb8L2eYm49NME62Ecx7zV9ATwFj5khMkggD3f/0mHDkwjFWnrEPSjaNj1Qo00glEU3ERx9ALF2tFPP/bv6L/5evx0IMPSpgnFNLOFF2BWFRZlQh7KnlRNCg7opfGbRIx2zpFjGr5YJkYazjgeCyKbCojldpzL75QWsiOjB5EdXQj9u/ei0qFI4HpHrT9THlZ8shKNRG3an5AOpFjj3UzCa6jd5VESvUvwq4YTM4HsXT5Uhw8Mob//c1hSZQa9shBVhrDJt7+ustxZHgvygU2fpgRcWaWiXyur22HNHL5kk2sh0rZ2YGEEmSRYul29C1Yiq5+ygaycIIKPvLRj+GBZ3bAc/WQBIVXLw3nL/W2JlKyLuC4+N4NV2Kg4ygaFT0yUKbYptLwY2mZSsD2PhalxqYCXP/53+K5veT3qSbUqMo2wH/09ffY3f5bVI4GX7d+ZoRVekzk3Ki4OVxtc4S5NjkLZZRp08jKaWDvuOAE+FLrcKTBRCliF86mjX8L5ZDPss6Tts3MMi9bjq9T0C1KumoNP33fR3DsOWdg/RWXIokIhp9+Bod37pNz6lefdzYOzfIIxCg64knc/JNbUCyXtJBiEgkRzxjOVabC0gdKaPEQeCo75RxxzY71iDxlBXRalByl19JUcExcBG2ZNHK5LNLZpAyd6c9VsfPZBzB+RI8mCQM9hk+6/eUUNQX50sHjUSDIA1lDma/IhZGDdyVp4zWYTho55Znjq+coxJNOW48nNm/HzXfPahMxN6vj4dKLLkB54hAKM5NSLOGEWjYPWbqNUEk7rthlRANVRkLK4WI3Cl2E75VReAmk2zvQPbAYXQNL0N3bjxdfeBYf//TnsXt0TPT/4vVbCfyc7mW+walxOOhOBfjl967C1KHd8MiPM6KY4wSjiQSiiSxiqTbEEhn4bKIOfanYThZL+OAnfo3NO9nn67TK5v/Q0q0Gfd5/alGKdRhzXrhh/+QajZdv8f3zfs9GOOHy5zVyW5zOl2ZjHl5zykIkYzpYSAzfRErnyYfvDolhbOc2pbZ2IKMNPdR/NxwHRx5+HBt+fjve+KVPomQ+UErefNPZIvZueALxRojMsUM4UJvF4488ak7snRPyiDZFSrxWr6JhWaCB4betDpwXqif96tnplnqyzIncSMRHWy6DBUMDMorulFNPQn7vPdj05CbkC1Wp0skZOnKMChGHFkJEpyxG7CGe4DXoURzi1f25I7NdKV7N0ytLGCW8cXHeZa/GH++8H7c+WkLgxtCWSeGSc8/EwRe2o1rV660bWYEjx1+xAqeyCW7qeIzGyY2lg+rnK1htTsJr4oPNtXUi09WNnqHlWLJsJR6+5/f4769+G1P5RoublmTL0cm55Iv1SMYWeIDnRHH5hcvwT5f1YvzgfqFO5WwgyjhieqRMIpNCLNWJWLJLmjCEN5cJBhohKKYrVUL86wduxnN7qxK9ZcYJPTw9NfEwXCxbcQwmj45hdHwSEYeKRg6AMkUdyUv+cRSYs21tCrFf841/vtGruC7EikVdWN2fMqfJRYXY4NQ3IgJn44a7Qkn6iAtbs/l0piCNXNrCmjy7voRfvP96uh5c8ckPiRiZHDCxNflizjLkkSW86WipjBtv/j7Gjo5pVmz6CSW8WLWaEuaKmQxlJg9JOFbhiUQjrR7KVuK0MicNv6ZARIPhGUFMcGeqdbzzmmvw2O2fwq4dwyjKNF56cgdVOUyVybU5Ntwc/Sf6bWLzCE2eXpotZ9oFxC9pohAsPzdqgYUo2s+Fl16EX/72Afx1WwNnnHYyuiJNcLCRDs/XJIk8vayrESvRWzNacSPTyKgCVEUhjckYgaHaNIdQA2NfadfAILr6l2H5mrW47Wc34XPf+bk0f7Cxer7RWFbIHoFi/++Wr1+LxNTjKM3O6sP3uVkjcgQhhy/JIbCxCDJtfYgmu+QztXtBE/IWA8KurEoBdz1wAB/7wq2gZtN3I/ji/3wKp65chtLMCBq1gp5j5Cfw/P5pfPHL38TEbF4cRqsRQpSNc1hczh+VQGbyL/O5LT7fJKet3EU0OyFSUeDdb7oAnemkzuB0HZTyhdZRjc72Zx4K6b3nhwF+lMKCQJooUpk0vMPj+PknPoc3f+ETSAz1IhFPq7A/dOUNZ0ZHcf/tf0D9yCSu/vD78LXvfAtT+VkdrskZ23U9rkMSSBq9OZpDDJzezUw9siJ9PVNez/ax2hHePzcJpwZI+Zg9qYkEuttzWL5kMZ7cuhmf/MyX8PQfPondu0dRKasn5YwXEjL1RogKoVejhpjPPs0k2tvSiJJW5IgD6e6WA8JlPeSYkyqLOhUUavRgVM0xB/CQi0Sw7rR1+NldOzBa7MJZxw9icmpaey5FNalDMptUP7YKNIrx2VIotJ2ncIVuUOb+SUe8lq45/Um8rKmuOm4UHZ2dGFyyHMevPxU/uvFL+NYv7zHFNdP3N0+tx8ojXM2REtEMHrrj37DrkT+jYvIsXpPO1vERift6MnV7DslMFolMP+Kpdp1eIId9zUlsRdvi6AYeGz2ILc+GWPfKq1EceV7OXBUlp3gr1RiJ05KGkTb4qTZ4kRQ+94Uv49GNGzGd1+N2tGHEQ3d3Oy545Svw61tvg5w+Y/KuuZY20/xhRE78+SWXXIxr3nEVZkZ3CQHCI7tVhBjAk8NqAeepR+8OybuyoYAXRK/DzF0ekBkfzMrbHV/6Jl7ctAkf+O2PRe3nV+vY+uCj2LLhIezftw+ztQoWn7AKp5//CrT39uK2X/wK49NTAlcaDaX9RHQlwy3N2e2mY4dJGrvj23IJKY5QOisVSdtRLgmpJAct0RHnpxTLVex4YScGB/qxavmxeHbHNrz3P96HvY//AC/sPIRKFdJkzAO6CjUSYQ6WDHUikXSkiUA2F43b4mWdxNOSifIT7ZgINnY3Ak/gwd6DY1gw2I61qxbgtw+M4p3v/iAe/vPtmMoXTc3ATCXgqDgZ9KMnNBOREn/Ti3Ktk7xPYZaUPSKUsc7GdswwiMnICtcTznzZ8eskum148H78+M6HWke66Dmc+nBlsq4HJBwPb7r0FPzrG4/Brqefkj5O60VFHMchmlFPjDyRTiHVlkMik0My149oPGeiLDlqnlA3d4guoQd/f99zz+PFPRNYsuICLe2rIN8kwHMSajaixxOd8JNZeNGEwAi2MYool3+Xw3TjUpke27cVt915H276yR/EkdmpWfq+qhviGvEIzR/88IfoaEugXp5BIFMbdKqtdDYy2nMMH3uQn930oBynYs9gaW9rQzFfkMGf3V3dEj3GDx/Bd655HxYtGED7ooV49rHHcKScR6anExdceTlWrz8R7T29cvhrKDca4KYvfAX7Dw2L163WGmLksnGoS5Hh8qHML+/vSCNGHEfcJw/fhG5TsVIqT/Gq4DLDAklLlfP/6HoPMDnLsgv4zOzM7GzfbHbTQwolEEINEOmC8imgNINGitKkCiJR6QKKFEGRIiAoRaRIlfJRpEiTEkpICOl9N9t3p+z0svNf59zPM8n3X/+/Xl4Jm92Zed/3ee7nvs997nOCGE6ksPTLZTji0EOxfv06zD/xGMTXv4o1a3oRHzGp6Uw+j1nbT0U0SvYhp3lqFLW14NRAMoqxb55Ym9hX9d5DkicRECgWMJCuoHtLEvPmzcBLi/I4eP9DsGndCmSypkOiiSeXpmXoo+l8K810izWG+XNG+adjYhpnxGHk26pk+UZR0FCuY+b/EC8+9zQ29w3j+Xc+0X1hXdJQX2+FuiCgIr572M6Yf9h4DG1Yh2J5BKMFDjmXRFFmj8LDlKFIDeqb6lHbUI/G1mY0tIxFXeMERBqadYoapmiLy7Ma2bxiOrf686Xo7i1g8qx5aipx4aoK0ILcShqzRd6GmvpGhGsbbCyQQqvslQjV4SYGBjpXI54YQG9fDGdddL1ou6I3u9PNL/LpM6bjr/ffr/tVysUwWkyjmCVoYkpoTCfVFZeZQ9GaQSr8iG5wqsb5r9MQqZDJofvjxXjzpZfRvWYVou1tmDlnJ+y+795onzFDxK0xnIKh9Z4YeM61uAI89fdHsHLFSqTzWc1FUm9F+oCFAnaYPgltLQ2oYxRxO3PbLpWvtH1jwQ+qekMrLXbHS+bm6RkcQlNdIwaHE7juppvw7lO/xLKl3YjHMpg0uQOUa6kVisIC045pbjIvtuO7P/9v8M1LInDdsKPGG0fUKZMpY9yEqRiMD+I/S0s4aN99sbFzg6BKGz1jJKeR7qjUBfyG4cJiMGGU5meoi9giJ9zFxSl3NbWi7c/qonWoxLiJ4zVgvWrVamzsH8LargEEOAjBlVhI4bgjD8Q396hDrn8tcllqthQkdOQ7jmqMWJ9cf4aipsYQrQujsa1FIkr1Le2oaxqPcLhOqYpG8Rykyj6IEsayOTp//PobCER3QNvkXXSNypUrW4vUrXVCADW1daita0O4rk1IXCjETWdNG96LdHIAvZtWKE1etnIdfvXbe2zIuSo3Tf3MMG6+6SZ8bd5cVMoFWWFWirSQEafEgmCFPQd2lZmJFFRLBpZ9/q4WOYV0TPPZVJrGto/F1Zdeid0njMdOe+2OfQ7cF509fchxjnK0jGi4TrzqSCiiKRzmdLK7dtDjC08+hVUrVmA4mUS6UJQNR8fYDuw4pQ3hiB3VnNwgl0RFV9VdYJsjz8MN/1/dMCIkpNPmC/K+WfT5EkyaPAU33noLXvnrhYjHUmhuaTDLEqUJzBGdAqqMYG2oQMefRyBYFwihMDyX3+bNsi/T2uZCZmp38EGH4OkX3sEBx16IT997Hxt7elAqmH0JN0KOygEwhwn/sG0RWBNKKlgO05VVi0tXDHkhMuBGt7YpKk8963T869EnsbG3G1uGk8iVR7HX9g0484RdsHH1SoRHKUJE3gddPRgHrGhWCqZ8z0NwjpMTMmChrqEWdc2NaBnbJplqLnIqDTBFoWCRqW8ZBVZD0zyN8wW8+Pjj2P2Ak4GaJhZWFsH9uLwfJdRBIBI+onXNiDR0IEzacKQe4RCxbLv2TWsXo5hLCij4aNFyXH/7g/9nyJmB4MmnnsSUSe3Ip2mDmddMgIRqXV3HZ8pgRKYo2aPpZAzJ4WEEln/xvtIVHhvyd3cXxEqbR9LgIDFRa8Wb429FVbgx6GqQSCT1c3xoLFI5TRQYHcVniz7CG6++iq7uXlEpZ8/aQZGLI1Bqwjh80ttQW7gzxEtFnwoIm1ZX1JHHqDOg0pSQCd1QyCedymBzdy9K5SCuve5ydH/5gIkgSTLDmkAiEaoQtIJ6W0iKx5s1nf7vwrLFaTuNCA1/hwMXqVQeu+0+G0++8gX+55iz8fYbb5pEB2m1HJSgZJ08R+skm8dTMeqaWxJucimYCiuHLjDvzebyoD4ihZNoqyjtdM1Sh3DMccfhy8WfYtWalRJoOviAadhluxBGtmwWxdh3gD3MaiCFHd3+njrKkoMFGdUpQhqRcH1dayNaOsaioW0iahtaJHNn2u0O3xeHpWRDyIEA+ru68eHrb2HOIWdbse6ek0d2tkKBW/9WUxNFbX0rwk0dqG/ke/C0CCE53Ifh3vUKlpT8e/a1j/DQP56tNrYqNcCuu87GIw8/hHJuBOUsNwMFYLeedt4EgPJ9nEorF7KID/dhsH/AFrkWsHIYkyzgzeCQBLVLiIsyyVfu51RuedfMkcLYfq2trboS08mroGaUUhRp3PfHP2HchAmIgoJFNjzAyGD8aWvR2lSQo3l6Uo5DYLQ4vXuYhl3dLKIKV5OJoA1JIp5E7+CwSFk//8U5CMX+YyZMRDpIA3AquqIesJmjDc0/nfUHUxGn8afhDZdCGdJiG1uqADoVSxhJ5dDSMh7PvbEOs/aYh03rNyGZyWroYuL48dZtq/JgyOlhQ8da1bb4rPPrDWsDZfceTqORqUuhaD7xazZs0GD0gu99D8++8BxisR788foFWPHB2zKPGuV0uYcp3Xr6v5jy1gFjj5kHIjYQzUDD/1EFgcjKmPEdaBjbgbrGsYqyXgSWQUfi+FKaryAUDOGDN/6D/r5RzNzvuxqEMCTFY9//F9KsDpOT/xWMoLZuLKJNY9VwqqurRfeG5aaBT138fA4/Ovdy5Ecjii92ggCffvIBykWaQliBKTjapWLbkrl4taViBulkHLHBHkG6ga8+e7tilEx74LQm5BFL9yxDvni00hqbVnPmV0N8nEc2Hxp5FPwg/IDWmbTcmw2c2OAQ6qJhbFz6BeKxAaTSSddW38biw7EYjatgT8lPpRu70Xwx/ZFvF1SD8mhekTOTzmFoOIb+ZALHf+8EHLb/vlj/+V+QSWY0n2iWhER3jLut/FqDFIa5+2l3nzd7Nh0njywq2iS6J4YVsgX0xUrY1FXAUKEJe3/tIOw6Z1ekYgmlcrxHnPOslCgGZDOmkopw0+RuzN1OGKm7msSGNoC1l+1EdZqR8gDaeTZ61m7GB18tw19vOxmLX3vRWY0bRcFvHjuh/L1y4ppV2bhtRsREZ7D6hCmMusZtY9AyaRwaOZzR3IbaSK1ZMnpxFj0YUl5L6B8YwvsvvIyJeyyQehh/jlGfr8YROKqKVS1U1O7mQt2qNBCooSpbI1rHT0N2JI5UKoEMZ2PTGcTiQzj/ijsUDNno2W3XXXD95RciUmtNwVAN01yDlUUDUSPTNGFUmhRyyGVG1IhKJ+ICPgJffvKWIjkLAC5YSh1zB3NR+YXMv/vmCBccZY39sajd53T++HfN8qkjSI+XEN55/l+IDfQ5rRCtLBfJ/G63SGsphWvUlM2dmF+SmNCAtWeq8UKK1NcEOaB0s+jqj+Nbhx+ISjGDaDiPptAmpEcSzmLcpSa+gKky5Dx6YtJn6sS6NMZyS/sSh10yF6MoFioYjuWwuS+HbLkBp190jdKlZJIQltk/eqIaE1fxddymZ7HG+U/qhEsagmhTmQ03aox7D1ArXFXwanKfGH0e3znuBNx0y62YNaMeB+1Sg5Ehs7thu92L/fiF7jeMTxt41Psoa3wdc2ewRc50kJB2RUKkrZM6MGbCZNQ3tyEcrTdXbhrgOp1D5rocZPjo3fexdvlGvPRpCY1NTQqM+fQgotE67DhzO8ycMQ0dk8dx5Lyq57P1GdqEPslsE6bNQl/vFqRTSaSSMQzFkrj2pnsRrG3CH/5wEya2t5sqQJnyeFSlZ8AzrrvqDM0KZVEtAAAgAElEQVRxGiRL4p2d2HnEhwaRiA1LfUw10cov3qswUhtf25waZDcoGxBGbdOn5sL2LX/KP5h/jdlFq01eKqOFxCEKvmczqtoZrd544RkUsrSfNh0PLR43ha+oRQdjFXxGT2Uw83RW25kFRRXewEi0Fu1tbZg8eQoWr1yDO+9/XF00Yq2/+eVF2HuXGezFId7zLga719GByG0qbiwn7mPlujUa3AS8ik2vVOXugwoalz7wmpiLJ0fy6BsqoKu3hJ33mIdDv3syCpkUUumUCndSjcX5YWPHDsEq9EnM1/oQZuvNf2FXmZueejE6bbJcuOYIUWaRx5NgFKiLhPH4M6/g9msPxdpPliAju0hChdbX0CizI+BTYdfkn62AJi9ci1xENIuopDvb3zmrSg4KU5AatE8ch9aJE9HSPg61DXZC+6ktXU6wglh/P9544XX0JWvwz/8MVgOWXztZaqyPltAUrcH20yZir913wezZ22NcexsiUQ40MK0JoX3iDKSzJeQzSQwO9Ei1bOqM7RGONiKdTOp0i9RGxRZlY4mU50gwJIv5dDqBaJTTVGaiZQxtk7lIxuNIxGIokG6dKViGsWrJf7XI+SEVHZz7AW+6ZNhYlIashU+ExFtjSLWKJqM1QDRSi0qRWDv0wMnFEK6KED758AMM9na7QpKbwQv3UD+wiCI1vsNBTJ82Ba1jxhoTLmpy0T5N0UAwxeipshuuVSoVDEXwk1/diIHhQUncsUX28vNPSJmqQCkHN1BbzGZx6a8uQmN9EL+88DQkhjYhEesCygX9TE3QhhMMAzY5NmIw8vSsCaFYNKgxlR1BLF7Chi15bBkJYJ+Dj8eBB3xNmDTvi6gPOdMON1Vo77dp2oJWQNuiZO2jNEzDC7bplYdzqt+lNYzwPCV23W13/P2ee9DTvxrnnTgbPRv6nTD+Vhk1Ugf8F+cnPZ4tBM4zKQmdhk26gt1lyXEIETGKAv97zJhWjJ0yAWMmTEBjKzuetdaR1Zepf73+wusY7hnC60tT2DRsNuYeNRJu4FJcno0MfOyJZFMjaGgI4sC5u+LA/fbCjnN2x8TtZiE2MCgTYZqS9XT3mYComkPqWGi8keuICmXk0Mv5jdY1OS5eukuTC5/TRuB153JpDA30I5fNWX6fzQmACKz58oMKo4B5H1IEJi8UgwuJ3+eiNgYg+eYFHRn8MI21zG957BaE/SbjCWltcMOEOFnCaEQilrS6g8rbqJD6j+f+F6+8/F8Uc3EsvORnuP62e/HdIw7CmScdr89AfUE2Y/i7cmzQgzd2YpYSEzlTx6qrjeC8q/+E/ngMrS1jlWY9+rd7MLGDiloBFHjDKiX885//wr9efRUnHn8sjj/yGyhLS7uM4086D/vP3ROX/fxsSUDzgav3X86jWE5iJDaITCKG7p5O9PX3KV0ZiqXw+doYcjXtGN82DlcuPBuZ2JA8SbkRqNjLIs5SEfPsIaRYR1MuWonzhJRWoxliyTBL3GfTd/SNLq6TfKkoigAtxB95+BGceexMpIY2IZsqoCi5OcvFVRQ7oygtdQ4CODkGi76+KCSq5VIXktEcnOn59FysrEMmbDcJYyaMR9O4DjQ1tjgukcF8yz/7HEs/WY7c6Cge/U/WmGz/P182VOx0IHnCUeg1W0Q+l8Y777+DWE83Whrq0dXViZ6eXgVUpkb8kLJeHzUdeDFjaWleXy9Yk5uOhsHhWrpCFwQu5LJx1AYLiCeGkIonZCxGKDuXyeDzzz5HYNOqT2VxyLSgtbVFO5qrn1/qzgWDSI5QUnhUTsmcjmFhVd9AxdaAikk+QLH5olGTNpCOtQniy1HZGVHxoT7z4ht44l+vIDeSxC9+fgFuveMeHHvkt3Dmqcfq2GEdQPtw1QUV1yV1pkzBcFQXGKEzcLQRGzb3YuHV14o7w2jSMbYVD9/75/8DD5527gWIJeK449Y/YEp7qxZ/rlzGSWdcgJ9fcBb22XMX5Y68bn5mbiy+FqNBLBbD+o1d+PMDDyMeT0ioX8zCEj0589h/7u5Y8N3/QSmXdgYBHKawekZeP5rfNOH8RDJp9zREMpxztHA0ChZ39FJis0VT7JVRpFNpdPf2onvjWny0aBEWnjQHvb39sjgcpZ6868huzcVNtoM5qkcbhFq5ha0T2PUkWKuJpag+AT+TlYmMjOPGd6BtQjsax7fLtp2OzhQU6tzYhQ/f/ADZkQISoy14cRFV0P4/mISOaag01nVu/UAxWaInn3ISvvvtb2Kguwe9XZsxkoiD012EniUrQgoB0z03Nug57kxnGxqbVeCSMWmGAzYvTG5RuZhC75YNGOpZL1cOpn6U8HvzzTcR2Lz6s4pG16qSD1YUqSFRKakoiJKSSevnuqjxzrMZKwZrgujs3ITJkyfrA3KzGBzpCT1upAvU4TZ7v9fe/ggPPfEvLfLfXnMZrrn+ViyYfyROns9FbuNlHNZgrkXMmPAkH15jy1jRBnijiKqotRxuwHE/PEkQ4llnnYWHHnwAb7z8vCwafdF6wg9P1SzjYw8/jAYO5nA8brSM7596Du645Xdoa6mVozSjCFMiRjMueKZdjML5YgULr7pGgv7nnHUGRlJJbOnpx7JlyzE4PIzmxibU1JRw0jHHYPp2kxEJ0BOHC4aLHWrvaySQVitNTfpv5prkk2vKSRGfeiUUI8rJMHigrxe5dBbDiSRWf7UaU6fVYvftapDN8PhNyQCB86s1o9Yp5UC2kCIFFMvFpV/CjUDpPx3zjvchEMHovrVigJLSamuK9OfWMU3omDQeYydPQH0jyVoN6Ovsw8fvfIR0qqL78Z+lwxjINQoGdplM9Q8NL25LSNPwiQXM//nGN/Hdo47A8JZObN60yWjG7LiS5ktDYUpjFwwFo+UmVXw13xCNyq9J/B3SF7jQXSotCe9yGbWROiSSMeHoa1cuQX/XOkmDvPPOOwisXvp+RYMKFLiXGW0BgQJ1+ehVk7VoTIcxcjBUwFiksKkMq5QZAQ27cvOaouEW9O++idTUxEImgOdefQd/e/Rp5JIJ3HL91bjk2t/hgtO+j0O+to92KSGhOppEEYVgoUIYhRAUtcPdWJRHMOj0/MvLrsLqDV1Y+Itf4Jabb8Dhhx2KX154gW46c9X5p5winfFn/vGwk/UNyqtnwenn4fEH7pZ+osnUuaED4vajoxqG5k0aGhrG5dfdJMbc76+/DsXkCAYScYzkcnjw0Scxc/p0pXaMHqUSq5AivnHwPOy/x26IhEbFxykXK0hnuMmDqIvWVt+PqZnVPBX09/epeVUuc3glj0JpBCef+h1Ea9OWlrBg1f+ZLtrzSMcoSZdCNpkS30gggU+JWPpoJNHorNzcdOlg/6BUpu13PaK1TFGCytVFOQ4ATS11GDelHa2Tx6JtzDhsXr0Ra9d0Ip0uI5lhDVaPZz4ZxmiZ3lJukfuWvshtDrVyc6p8Zkd885s45Yc/QPfG1Vi3YpmUBpQic0Cjlhqc5tjhIUEOn0Rq2SiqRX1dk6zPqaJcofASDXdD3Lhhx8+3BqGpLUDuIPR1LRVyWPbZe3j1xecQWL3kLbm/jWY5rV1EuNaEJMUzKVrOx+LBW9CxqcEbpfE4MhedWKa5dpmGNvMoRkY+LEMazOeysbEJ7yxagjvu+zsKqRH88cZrcdFV1+Lqn/8Uc/eYo8FiFhDRxjFaoGKQgXmfEaoshXKafZIRDmJzVy8WXnaFCrbjjzse/3j073j+8cet8A0EcOKppyKbyePlp55AoUwIr4RMPodTf3IhHv3bn0XWkl+Pe23Ln03li7lzPJbAldffoqi98MLzsd24duPhlEu44trfSfR0wYIFeOaZZ1DI5dAyZoyYj8atK+PIww/G3jvvhPoQIciCpof8Zi3mqfhVQMBpqtNNj8ZjwZoyTjnzIBO8L5kAv0GvViBSZoMPlJuVKUeFXJl83vL9fAGpJKWuDT4rZPLIy3qmWCXJFUfZUQ4gwe+XoNogGh1FfaQGjS11GDu+Re4W7737KZLJIrJZnkS0lhxFarQRby2J6fe94n4VrlSq5WDKUAjzjzsWxx97DAY6N2LDyqWysuRpTXKWOPW0inRpLhe0Nhprw2AQdVJhoFteCyJRYuO1qKN0NwIyY1OmoeEXP4Ngolck7andT3MGdpFjfQhsXPzviorEyqiOMEtFuDMsovGLi4D+lF48Xdi1CFd5s8qm5babFOJulDwvbbTr602oXlCcGd+u3NSPW++6H4V0ArffegMu+OXVuPPWm7DzDjPN2luzlFYtG9xoeDPvnhVZZtDkKaXMzU486UeIJxP411PP4sQfzMevL78cc/faE4VyBWece4647P+4/x5NsPA1aMp18unn4u9/vctEfhhNyZsul3V0GiHMmkapTBp33fsQln61HKf/6FTsutN2BlvV1OCpZ1/Aex9+gksWLsQ999yDRDqDBSeeIDZkf/+glHZp5Ugpt/DoKHbeYTq+tudsjG9tQDTMBlrO+BnUa8mlkUyk0NnVjZ+cfxzaxxufp5A1tz2mJ16ov1Q2Kxb/RSKYcZRsQIV/pw4jA4tOYYqu5gpCGxiAypTsyBflkl0sBdHXn0AimcP48U2Yt/8uyJUL2LyuB6kUZe4qcrVjoKEY07srM+hJmMKApwZLwzwYQH00goMP2B9HH3UUUMlj/erVyLJrnorrs/FSRUhzhrlUIlB+TeJabVSbjYue0icMiJE6YvX15ptEtKWRJmMV1NUz6jMlZPHpbGDcXHANuVR5ZiA2t0DYO7D201cqzEO5UPkNVrnM7XgzeIz5ljujmm8gMJKzQLIGDqWALWp7Vh/vv1/o3G1ECZg7ERZcvXEAv7nlDuSzaTzxyMNYcNoZeOzhB9BUz1zYyf06nRNP1vcwFd/X85XVjHI0hBt+fxs+W/wFrrzsUi3YG35/Ex5/8CGsXr8eN9/yB0ybNh3XXfkLcy4LAOlMHmecfT6eevQBVeLehUxdUdlyh7SpuVHThQzWrO3Cn+68E+0dE3D5xWcjo9QjjNFgGBf94nL86Ec/wlNPPYW6aBTnnXE64uzgZXMYisWwbu16Se+lR+gNVFGkZspCAdIjD94Xu2w/BchnkMmkEY+NoLO/H3fcdQHCtSFFvlIpIyqCpq4c1MhIXnVMc3RYX/x7K0R1nzXiZzUWH7hszgtF8UOISlSyZXUES5USwpF6tHe0YOVXq5DOlMBbneXAiDqvZv1CKsvDb/SiEiIZL4Dpkyfh5xeej3I+jUwyLhGp4YFevW+IsDLlQ7iOIlykhuxwzdRG6OIHFZw0DmOAjNY36J4zitfWNUj7MVLXoI4qO6isBzlcrY67716709ejTH6w2QRKDYhUJ/2jVx+pjGkdg6JrQ6taL4+qk7V69Ur541Stqj2nm1GDhY9rDTPSW/Q35zU/g8kNwzfjvysoV0YxmKrgmhv+iGwug6eeeBwnLvghnv3nY6hxUznK811Vrg9vvygYUXOQwkNzrltnRK5sATjjrLPkpnbfPffiuAU/wDN//wde/fdr+McTT+K444/DUd842Lw5g/QPyuDsC36GRx+4x3VuHQ2YprGaYqFtSUWRsEgia009Lrr4EsTjSdx3x026RqUO4Xqc97OFgg25ITilcsDcvXUvUyMjEhzK5UoYjMcxOJRA5+bNWLV2rYYfrMYJqaPX0NiAfCGDkWRWKMOSt25BKESYsYwRDkMTFMjxHtvQgzU+rBssxqT3y3EnpqEq1lEujZq0s+gJfJ1iSTmxmlBFLuashJZWr1iDVIrIVgmpDGSXw7diocy6iK6Au809DM2TZmPL2hUYScaFrHnddrJw+TnCIVPwMuq/zWmSaWpD4dbFZmteLEx6I42O6v7R/Ff0YxaW4ajc9BjJo/X1qsdUPGujmQugwBE3muitZ1SvyMWCn90KfiJZgS8/eLGycvkyzJw+Q29CrFptds7n8YhUty9dnf8kA1FFXZ5uwcTUg9WpIjs+imIp8lTIZdNVG8Bx4ybqQw6mCjjr3J+qW/rUE//E9364AC8++QQKpaxkBRwRcatr8DYDr7bovXyDsw9RmkQ9xNOR4Ws++gje++Aj/Oupp7H9zjvhvY8W4YG7bkek1mgDzJUTqSwuXPhz/PXue5Q5Ux1AN6hiXqGRcK2uw/+fi33hldcKBnzkvj9bGqCUrYR3P/gEr7zxlu7B7bfcqLyYC7hYzKlLSwt0/vxIJotPFn+Jjz7+FAfu/zX09PQgHo9rkbEAE18ok0JDtA4/Pf0InH3ygRBkGiwjPjxsBgPFvAaCGR01rqdrr1FzyNuJ+4hu+jROz9AZXvHU5UnFHmmQM6gA0sND+GLRUmSyZeSKwEia+o3m01pACLvucwjm7nMQli5ZieH+LcbEzOec8oGzKHSbTHWQgpQFI3GF+MWGkxuqtlzahjZYdDJqk+JdEw6jsanZFA/C9WhmM4oiSs1E10pSSivS5p4pjReeApRe6oRnb0H8KaNpeMBE2cVXn75ZYceot3OzdvzUqVORGolVbQMZ/Zi2+AfO6KxjoVgymzqNs9ki8RCibwfny0DHuAnqHxLa4o6MJ9I47Sc/UTR+9smn8b0FC/DsY48iEDTDWYtC9gA9DGiojhMvd97t2mjcqZKpKOOt9z/EPffeh4fuu1fFFzfg9b+/EZ09vXj4L3fbKF2AjdGCpvaff+V/MYvikeM6dExqkMJNpdP5wXgdQRV07DwuvOIaLfI/33qj4CueKvKirIni0ssuE032xuuuFvWAr0UEZHiY8hwUHCJUWMHf/v4PbNrchdN+fCrS6QyGY0l5NHVv6VEakxhJo67edBM/+N870Vg34jxVR5FLJeWLlM2lpfe+LXbnh0qMM+4c3IxZZv6fzqnay+IRmm2M1qN3wyasXL4cI/EiMtkKMrkyMgVjQFYCIfz0shvw4bsfor+nG4UCU0Xn86luLrk6ngvjjKu0nreaWPmClM58dpTbQAUXIdeVLWrCtxHNI9Q3NmkMj02fppYxaGppAWpqq/opzNWVabi0xw+Ha9LMcZtMh8W51Ln6JLBh5UcVeTcSSkMA3Z2dGNNSj+bGBhVCPBr9MSMtaILwQXMD5u5MJGLKrZgLMnIxb6pjp4zQo9PIZuGnwrSmBqlsAaedfbaw9Ccf/yfmnzgfTz/2D5Qq5H4zlw/JF9QTwLzNh+YMCXUSJmJu6UYdfAHGI+vHZ5+HKRMn4bqrrtIGPOdnF6pW+PMtN2ig2DTFLUqxBrE0jLBaBoODg7rZLHhamltde573xZyDn335Nbz677dw2803oiZAe0YbkOjsH8R9f/krWhtq8auLL7K2Obu+tTbtX6YwP8fhSgXccMufMH78BHx//gkYicVRKJFFmca7H3yI/qFhFYKyVsxkUBkt4IN/34LGKIvtAEKVUYyMDCGbTaBSKmC0ZEPaSp2CRvBShzoYdnwgAwAUSL32IPe5Gy9MDcXx1SeLEYvlkEyzBmMaWESWsmuVEH58xkIsWfKF1gDvJV+bs7r+ufj7rkXL6F1FvawgrtrYuKEPG4whqcpOYj4LrheC6Go4uaje1NKGYLhWtIIov8cmUZhEsYhzgeYGsZzbWK/bmHPpvSzgMgBZKlWDwNpl/61YEcNlA4wkGTGyWLViOebM2smNEhm32QxdCQfySGNHkxgr4ZwwWto75DMvW3GXExHeYnQn1GdF6igS6RzOOPdclv94/B+P4vj538PjDz+gYVoIsSHBqVbHEI9hOZhtQxflBdhdtNfzN5gXffGlV6KzqxOPPfCg3vdcLboK/nr7rYIkmUYwwppfjj0wL2ykhkItzXppH2iRxsbteMNKGIqP4JY77sXPLzgfUyaORZ7VPGpw85/ukK35L39+IQKFnHNeDiu35iaiWYGOztEKFl7+axx19NHYY85syUDnizkFi1f+/aYaTDy2991nrtKYgUG6UQ/h1WdvRjQ0Ih4QiZnx2CBKuRGNEbJDari5pSH+wYsazPlGd8Ly/fnv3KxMY1obGvH2q68jPpRGKlNBMl1EhhAhx/fKo5i2wxxMmTYLmzdvRrlkJzXb5JyH5Xtt2+zZdrH5YMjvsZ/CgKTF7aQmagkZOvFOpS0hqhI3CoZld5XFZ7SuCWM6OjTwTDNgnppMc8Vtd4iKUiG3JvicqzWjYF8aFAdNUmXU2LCBdV99VNFUifS+66QZQlI6C6dsfBi5fAotTY32Jk6DcGx7B9IpGrhG0NDSblxhx7DjgqiK4DstQ94kbhL+TDZfwo/OOgt1tSH85a67lSN3d23GcGwAE8eNV1HGytwIXkbx5e9XF6brP7BPaP9GaNJee3PXFlxx9bX44623Coe96JJL8KNTTsHXD9xXpENuTMJLjMDDw2xLA80tZg/O9/BDIYwwvJFcbH7ihq383/3hz9ht19mYf+y3tLEZfS675reidN560/UIlItWFMsivCRzWkJifCD82at+eyMuu/SXaGtpQiqZUmDhZ3nqxZeweXM3mpsacOS3jkAxV0A6l8faDeuwfv16vPvSrWiqI3nJOOeca0zEqZzFaXSKtDqilzMBsPE9W/xeJ1zQYqgGUydOxFsvv4b+ziEkUiX9P5UrSyA1X9JkKb591HysXrveAoL8nszjhwa8/mvbiK7o7Ihgyse1HL3UHuFYK9RrQwZEKAJXjLvDRcxMIBKpl0Rd69gOROobMHb8JD1TRnkGNCn8Mi8vmlQHTwApKTigQgiSRGct8PGzV8ceV37xboXfFGQo2eAwUsmEUSgrnGksYM1XSzB719lq9ISi9WL9BcN1OrLJpWAO6o8v/j0RG9Iu9cNjonzyCBGNt4KTTz8ds3beAddecaVaPcz3ypWiOCj8HIJ9eFHkKrgZQL63FmOZu9MKVM9W81YrWUbvn16Mo448Ct856iicc/75+Ot996Kcz1QxZtJ++TrSTc9QSYBpVhjsyPJGmRVfaBtEialZRjn39X+4WyfZNZf/DJSo4Jly3U23Ilip4Le/vkIpnzQdxZTLaT0QCSAHhg/kz/c9iKOPOgI7zJxp8nCKjGU89MST6Orqwbj2dpz4veME8w0lE3j1328iFh9Ge0sHXnv61wiHydGhAS5RlgyS8UEUWNw7iQ9PWxbtlTg5T66CPR9+sage3NKD1UtXYng4b2oGhYqieI66OJUaHHDgN5DKFEWVMJRsq8tHxaUaDEDqlejEM/KWWZ3bzyqldeKptqhNnpvXZf0XQ13kBysTtjAaGltQW9+AtnET0NTahqYx7ahXJCePxbrRfPaK2jqpnPY4i0zWQJrssmH66mnDSM7Z3lVL3leFYmmC5XBsibKoIx45WmQaMypifHNLi45NznWSBcYHTtzZi2G6cUhtDl4s8XHeAN5kX/VnCyWceNLJOPiQA/DTn5wjCI3TM2WnOssPmE0bpswmhNdmNLMCci4syjJyVD8v6bHcyYEA7rjnPiz6eBHuuevPuPDii3Hv3XdJY4XRSHUEu7KRWj0ULl5uUk70COWI1mLMmDbx6M3R2ei3cm8rF3H7ff9A1+bNuO7KS+QhSsTk1jvuxje+fggOPZC0W2q0WzdORSmvgc2XMnVlosjkaQKcRiqdVd5d18hOYxTPvPg6tnT3YnwHF/nxlrZVRnH/Aw8Lkz9x/rGIRpqw8Oz9lKOTt8OoXsomMRIfrqIorJmsGOfklM0FEBPnsyDpji4NH735Dnq7YoinykjnRjGSI4WB/PWAHC32nnsIunp7kU0ZYuFPUbvnRqEWJXab7rPPi03Sw4hipDD4Z+9pzNSJlGSE03qUipdLW+rqmmQhQ3GjtnETNfJX11CvnJyjeHxh4uuCDt1AjU4T1522moHu1FvrOa5PAQobV3yqFoO0QvKMcGarzWOgr7cbU6ZMRSsnNLzts8yzCNdYpPKOcfzTe0J6vxg2A5j+VIsfISKjOPGkU3DiCcfh2KOPdpxqi/TCN/Wn7UYdR1Sx4sNyeSc/Bz8fsWxGXUnckQzFE6FYQrECnHXuhbjiyivwm+uuwwP33mkqTVWXYMsxdZRrHM4UubjYlbvKJ5LjeyF1bFm4+kbYm+99hKeeewG33XSdToL/fvQZXn7tLfzmqkvFWZEyrkYBrX0vFp4b4WPAUGR3xCKeWKmsjRC++Mob6O4dwriOdpx0wnckabd42Up88MEi5cIXnX8WQjUBjCSGcMGZRyIaIneEdN4CKoUsUsSsR+LyMM2n81rkuUxaMO7I4JCIXUcd9x28/8476O2MYyRdxnCyhFwhgLwWBmG3IA445EgMxzIYGBiSxbyvf9REc2kGr5tcfgU2p0W+dZFXENEGI7ZulF+eipZD82T3Qq7Gf5J1PGUvKBbU1Iym5la0jG1HU9t4NLS2CW2xJqJZztiom/0eswPWWGTJ8rX4WQuymyft2elrBh2suO6rRRUuaC5ufiA+IP53LB5DY30denv7dKQzH9prr72qE/2avxRv2rjRvptl3TUbFvYejfwQviHEc+EHp5yK884+C4cccICaFVJKcovQdD5s87Dlzs0k//ogqqmMr+Q9qUqLSu5xnG4P4+yLf4F99tkHq1etwo2/vsK4027IlvWG5fusfW3aX//uvIx4+vBmMar7OoDFEUeuskXg55f+Gn+66Tfyu7ztzr+gs7sXv/v1LxAolxS1uYglr6aBi6LeR1NHjgtjebIdv5T24H//87mXsHFTN7bbbrI47yz+/v7YM4jFRjC+oxXzj/82giwiA2Fs6dyMww7dAYftP10AAYpZFLJxjMSGEBsawEgsqcDCpo6fF+Xs5G5774U1X65G7yBx+wBGclwURGhK8jJqaunA9O33xqbNm0U0E3eINRix3228gbiAC07wyD8zFZxucCNC/J7nveOaM3Iz+HHwxmveMPp6iNZbK7JAb24Zo0Xe2jFRi7yxuVWBhgFNp3itwddW4BqSwnPBzxcTHha1wTUtOVG1ad16BNat+ESYD3/QL0bKxKU54WfSBkEAACAASURBVOMGf/OZNLq7u7HfvHkSy+HuovmT7SCbnObKNMNTEWZtsr46M2n4LR8oKaynnXYmLvjpefjaPvsod1O+LhZfSTms/5IsBY9HHbscBTMHMWneuUaHx+R54Uw5uLA+WrQUT77wCg45YB8ce/S3zX8nHERZGuHmXe/nOYVMuPYv17qdDvZZtcFklUgkA2hqbMAlV92Ay35xMVobIrj0179D+9hWXHTO6W4hGLeG/J9MOlWliqo2cXIXPg3iJm5sbNbR/txrb+DLZauw84474fBD5mr+8e77HhRnfeFF5yBUyQsy5bUyxbrj3kfw59+fhwP2nYBCahC5ZD+yw3GpK9A+npMz6RQp0VQQy6OjvV205aFYGiNJqnsFxalnfcT0k8pXc+Z+G2vXb1Q32CNn4gxRd93fayd6qgaaNq8Vmepj+Ba6U7yikJOlex5OtNE7nnaS5nNiqgZaBFTnsV/R0NSCMeMmYfzUaWgd224Rv8aiPRe5cnFJhFhhy6EPuW8T5pTwkQVMThGVimn897XnEdi4+vOK2sNuvjOZSGhRbNq0CVOnTlGuPkpaZzqNdCaDvefORU9PNyZNmaoWs7eA5oI0nT3TotN8ZFVTxHI7XiAvfP73F+Daa6/GjjNnalJE7WfXovZHJKtuQVGu48lUyl7TpNiY9/tBay5IdlkZQVUHlMu45c57sdP2U7D3brNFTahTEUPusZG0yEnmB7Wq3JlC8YGqXWyL3Z9QHnfNplO47Po/4YcnHo8958zC5dfdiN9cfTlqqPNBVakQFyH7ByySihq04OloBVakOpzNa2UBRVSE7/f2x5/hw48/w35z98YRh30Nny9ZgZdeeVOQ32WXnKvCOZf3w96j+NO9D+IH8+dj3uwmHLBvEwrDvYj39Mv5jukNWZfpFCeLcujvG8ScObthS3c3EmmSskIochhFww1BFCv16Ji8ExrH7YS+/l6kEgktmnQiVm0A8lTW3K0DEDSZ79AUO6lcaqbFbh5BIm+5Z8ehDA8jSimtYpNeWhPyi2KXsxbNzS1obm1FS/tENLa1a5ETeeEGkGYkFzkjuQsYqh85PO7STyl8OadtwsErFn+Azz54m7orH1Qkz0xaq2uXirlGGmgpjzdf+zf23nuvKguRN3LGjJmor2swYpNbKJaXGZ7ivYNMitfayxbVzSHu+wsW4E9/uEURRgKgzPlU3HGz2YLn/3kjPGNNFyKpBubq3MXm2sz3o/QEtRt5fIv92NAgzJtUXU4x8RRg5c2Uq7ahUZuB9iDU6JNWCG2yHeZOnLy5ucmlZcxMvQqW5X5/e+RZJDNpfPfIb+HmO+7CLdf9SoxCwphMU7lA1MxhV4+dPIoKOekL2S46ajIXSYEipIEA3vn4c/x30Rc44vBDsP++e+Cevz6CLT0D+PpB+2G/vWZXfY6YlpHI9epb/9VC+Z+v74/GeuCbB4xBrncVksmCRHWoKJZJZJBIFjB9uxno7N4iFIVFf6imDrlyCEf+4KcINk6sSt8ZQmUDzjwR8ukRG9BOk1OTEF89leJJkNC64H3P58zQgEFASsNETTj5ROk3DWtwAsqisLaU80llJNdzVXORw9L8mRqpRTQ2N2NMxwTUN49Fx6SJ6r0wXeEaJQQqVQXJeRjOXsxnHS2aPRW6WocRjoaR6F6Pt197wajMm9csqTAfJz/FF0Xx4RiGBgbQ1tGKhkgUyZGEzKeMcG9FyKpVa7A7TWJrQuriGaTk4Rvbof7h+orcNM+DOPnUU/CXe+9Wx4tjdJRDIE2AXUehAxETHOL/VfRV5YuDKBMTV+RnemNT78zxeCMz6REz9uLmE62T6qf1CLCzmE/rVJIVtTjM9dWUhRu16sXuJ7ock9Vj/NXrK5axcs1KLFuxDp9+8RUuPudk3RsiNhx1UaNESlsWVfn7SpdIKnL/7c7waqH67seL8cbbi3Ds0f+DWTtuh5tv+4tqo6sv+5kKS3Fl1ISxFIEQXb6Qw0iC+i4l5ErAhrVfYN6uEzB9XA0yyTyy+SyaG+sxOJxCPFdBMdCE4WwIsQxwzXU3IEV1gUIWI0lSByh8ZF1CEqEyUlcw/kk2k1Z6EaPu+ogbDpEuT0Kfi1ApAwOLQE+m824ggmrlmEdD4Chqo6xVxIC3QpKMQ/4pHktE+Tf5+K1jx6FhTAfaxo1DXT17NNZY4wbyRSfXidr6Tpw1k00rYETDESTj/fjiv/9BV+dGy/3Xr/hMWoi8aatXr5YXOiO5xD9RRGNtXTXKqz2dz0t0f3BwGENDQ1i5eg2OPfbY6nGkPExNC5N+MJ8Y08lgtGPOxAGELz9dhGnTpmH72bPVTNnS1YUJEyZoKpsDCbzBvmPnoTF2QU3sxqKOQZ95DaxyEdAykFudN143moPWHKFrbEIt5TXccILwX2fZomaPYC9O8bDTGhV2yydmimBG+GGUYgc2nczyXXHVb2/D1w89ELOnd7BHbY2N2lrBj6pL/CYtWLfQrodpitFMDTmSmRGWrtqIF195HyefeAzCkTL+8vBzqA3W4JeXnIVoTY2aUnzIwsGr3pgs/PMo5UfRNTCIjz9bjk1bOnHIvLmYNW0SKqEw/vbIU9h5xnTsu++eWkgj2QzOOPs8tDaNRSIZRyFn+Td5NMxp/cAI7yUHqPnFwlzYP8EJar0XCgIAGDAioyV9Ni12MjY5laQpsoJIXHzexOp9CkoKCF+7rbVZEZ5BleCEGInhCJqaGtHc2oKmMR1o5P9byV9pRWODoSyM5FTv5WlpaFlFcLelwgx8tBIpYNmit7FqyWKEqPTKO7z883crxL3b2toUzdSlozgQlUZTSV0QHzx3IxePDh619m0XMz9iUbrb7nMwMpLUwqVlNQs7HS6eReiisnphTD0KOR2BpGxyATU2NSrNEKbuGhCGfRre6+SltIDYMvcFnJSpnIOzx6YpDMXX0QbI5Y0A5OQY6jm5pHx7a2vfXsuqdsGnDoLS1Lsrnu26oSFragKuXd+NRKwPE2g5KGZmAAVpZNtJx4FrQw6sOUQjAn0eaasENLtKHg3fd/nq9Xji+bdw5o9+gI8+XoTFX63GSfOPwcT2FnHPeQoYZyioWVned9Y73plh1dpOfLJ0hSbffzz/u2hsrJVg0f2Pv4DDD9wHkzpaxYYkX3/hFb82oaSiqQFI3kNpKusQjt+xtgjbkIMbvGaKZLJyWzevCHkOAmVUTmoBlzFayGhGl0FuhH+q2cdT12oF2bFkUwqQDJY0NhOUGAlj3LhxaG1pU0rZ0DoWDc0taGltE7dc00scllCT0g2IuEaTB01qa8rYtGEFvnj/XeQKtOi0/kxg3Vcfy8fTptUt4rCA4uJmGuAxSPMGCik/ZMHnSTvUGuHvbbfdVNx37734+mFfx55z99aH8ZFYPAXTQ6hCPKwBGE2JzvDh8+J5E/m6FKExFS/tQ5e2bDt9ZIgMj0lOM1nb2PGnWUjqQdlUvFrnqvKdsZXjwTNn58PzMKF191zL2bnQcdF7rUZKQDBS8HNLCk9T83wv24hGv2XXmFiNta1VGNF0VpQHZ7stJiQ95iVdpdqhfziJux98Bmf+eAHuu/9hFALADVddLLWC1Eha91eRTMQmMiQ5pJJTX4MI0OdLVmH1ph70dG/BhWf+EMViWhqJ9z32L5x9ynwUM3ENf5MQtvDy32oeks+Qm12TM3Tv2OZeKId2sm6+Rc77KYRLHG3i1GwRmrU66zTJUnO6SidrFqlUvDpCSE0eTkmJBarobikYT4Guzm7pvRCm5UnOzV/f3Iy28RM1CUTsnCiUKNBRcs7NPEDjfmpKWc+DIp/D3evw8btvIpPLGHeGkZ7/Ru6KLXIWQqYfwqOIaAVvJD+Mr2ZtuJdQjbkT89/Xr1+LnXbaSW/a0tSMeCyOZcu/wmGHH4bW1jFWGHLzcErcSQ0wEvGGcXcS27Tc2/I3/slFyi85szlTLEZE3mAxypWjWzvZzzZ6RpouKmhtX6k1Oc8d772jne0il7p4IqXFq61goyi46Xe36FVclRxH2ZG7rFll9UGYMFaOOSlxZVKObaxNprpOeZWLndGYrhfcvbaQbOSuUAJ+f99juPjCc/CH2+7GjjOm4oyTj7FNR3YhT9E80wrCuoZKGKRWJxWFx//1Nvr7+0UfuPyi05ArFWQD88f7H8fpxx+u+8w+AdOt83/2a10zrzOVHhGmPjQ06IwCDHfWfXaWjh5O1T1guinddDIdDdJlLq16RU1CCxL8rFHSQ9Jp1SEB0psLRTdaWTIELMiJsRSSyZjoxqRgcx1NmTQZ9a0t8i4lj4UyFAx4vIZIXdQGZxTNCSVWxOJk3ZIY7MKHb78pIVq56kWphkD6QxmBDSsWSXeFF82jy89zclqDf2ckzKaz1ZxS2iQakSsp1+SDFhgPYNWKlZgzZ45+b3BoEHvttbdGwrwZlj/+hVE7yJELmQvWoxu6eUXTgeGH9bwYcigYWYvOJMBj6aYNU1OVs7PFbkw5nULiPRvHwqby3XtpITtGoyu6NNDsFAnEtxGd1tIaXp9MnWCRmRs86Mb1mB7xAROoYUOIN99gLUuDPBdfn59Nt0itoDbrjldQCkTxu7sewkEHHIh3330Pv/jZmRg/tsnoCy4aiXBFDr/yXnteppwVxGPPvSlVATa6zj31eFQoqVsGHnvuZXzroLlSKBaSEQrg5DMuQjTa5PJka/cTe09nUi6NtEkif5/8RuZ9phyJGmlMJzniVst5SuP6iICnhpfJSGuaXvIhBbDPIhiSzbdcVvAiESj+POspBs+hwSEsW7YMO8zcHrN2203wIe3WW9vGVvn+7AiqZuIAM4NhqYTYYBfiAz34/NOPBXXLdVvdZsYX16hc/vk7WuTKv5wxLXeYGj4aYKWtXdoMQCO1YifaeJET/iFv12HstpttzM2nPjvP2lmiTkRSdIRX2/WmF27QY8WiujsOle+JQmk3j69fyGfNkcHh76au5qQxiLtGarXLCSXy5qlQc6/nFzsREKEfDtv1iAlvvvjYzNOlE27iSr74VfOo6KZPMjaVY6xMIxqxa8vo1VBXp6KIqQhTAW00R3flf/N60yMjaG5qVprAgorvkUcIN9z9BCoFNr+Aa35xph6StbSNr83fZUrHKOg7pqIQVML4++MvYjg2jD133R5HHHyg7lk8bgMbnK+kTAMjHn+P/z/j/CslmErvHg52MHAxdROd1hXuhmHbzxcKRuHwp6M2eNWShVJxlGS2DczC2/tPcSMSMeMC54gfVQR4TxqjUUVv8VzIj9I9T+vaPvvkUwWQ7590sqxdQnV1GNPSqsBaGB1FW2uLQBL2Dvo712OkrwvLV6xwi1qtLaVjJp3inFMo+GnwlD18NUPEL4emvC1X3So1Rh6zdd7SxhsvFPXAeWPJh5ZmuaA9G274atlX2GHHHVWczdppxyoq4gtHH8H9exiMab/PCXabsrEWv3IwZxTl0w6hGG4SRDef2hx1JovBit0zIH0uqZawo0f6RcxCRpvSFaOlUs4irorXgkGBJT5YRiPbmL6i5/uRKafF6OSWffS2BWKCqXwvPkQVpa7O8ASzdDGAm//ypASF5u0zB4fM2xVNDY0qxqxGss3um3ZWJ/D+ZLGhawCvv/OpFtNF552OaIBpTRp1dQ124hRzOnVld+gkto867hSZl4WDpqrABc5o7gldxLx1fcEa46BLKcEIcgxIHmrmQah6oY4ohqmmCTINhXVCMHCx3qKmIVM4aWaSuUq3EmYCZJXq3rL2s2dO0fw1a9egs7MbPzj1x2rzkzQnESHScyMBbFm3Gl2b1iIx2GewtuoeS5Woumu65TZ2p5SPi5wVtRfY9LRVfnhCeyomxEWxI4p/WjVrEgnEJX130Oe4fPA8jqwdXlYhwg7qySefjN7+XjVbDH82Apblt7Zw+H8VWeIc22khhIOfwQnxm4D+1krfQBzTv6a8mmcCKtK54Q4eMTxJvJ23URACNuQgBwtGcXu/YpEwobWOjdMTRiGX0g3lQuaiE8WYiA0XIZtWpIS66RwFC1mv2EnIn7eH4Rz13MCxwYhQNP79fU8jm0nh/DN+gEgNc1oyFCm4Sa615e7+tPWD3FxM7y9ajMXLNmFLdxcuOvd01IcK5gRirQKdMoWswXh+pLCIWvzoJ+dKOcxOrFEMDPTbyViy9FO1hdIic8G2wp6nOiG7sqjJbK5xc/Fz8Fr43HhfdPKpc2yMQ2t8FdXw489kCxktfHaQWeNFasJKUf395emycdNmfLlyJX581jno6BivgnTL+q+QGOhCd1eXGoBmp2Kbj3UYN1qEfzp5Zz9VFtiy7ouK8E1dnPFHCP4zT2LR44s0/oyPKL517cF/LxPBRUUclamF8lfBbx75oMaiQYy8iOnTZ1SPYf9z6o6qqeT80iXZZjwSFnV8bVJlRQtmdCttQw/mBJG43KaIalHdTSQ5PXBtEqYHLqeVYpebORRfw/2uT8WUB7PJ4Wicdn02xMtckxrY0uqLcIyO8m/0vDTNGl/Ic0P6KMx80jd2/OnDf0+VgNvvex4NtcDxRx6MhqZ61DuNeA4qqLilP1OtpWQeBeJ7Pf7CO2IN9g3249ILfmTOegGTBLH82fkD6bQqGISXyWHf/b+BufsdVOUX8XPp1CrYtJLvHmuDi9kXVABhfs+dyXvIFJHvJXDCpUI+K+D7qgZxY2j8PoMPoztfh89J3W03WkfmKU8gbq5iPoM1a1ZLWm/OnN0RiQSRGOzHQG+XcYvcpJGtTQMPqNNDeb4oXTTc8IidzhUEejYsqfg5R+5IXmCeTYJ8XhPSaWmxhJRj8gYr8kUi6Ovrw/hx41wlbsiDIrzcBqCOGLkI20Yfz1vnv5EaIAdgN8bkO3qWMlmxxiOOO96OSaN2MqIrbfF63BqVMbEfj2nzNfzm8Iq4OjkocO+c1HgnvKclF5rSHhWFjG5bG1EchNBcqRSZSCTLbW3MOP4MCzIxD0NGA/abSbUEMeKygxi5AKkA5YSMBMOytZTNoWsgjtowVXGbJdlABEGyacx1HbRrndqoJN7IvSmWyrjnkeeRjqeQyadw2c9+LDFSn3Z66QzPjPSEOfqwcjr/tPN+acWtqz8YGHidKkYJKTKV8BaTXrfFSXpbkWmFHdNVBkjCe6ybkiOUaq63iS1fl+hEjGjDNDU2mTa7z8lVl1kwZH1EWQuKyw73D2BL1yYJ9PNe+c9paZ655LEw1kQ+08Yg7R5tKstnBZLmWL+cEKLJL2hhFAsa+1f3aLTsuodW/HHB8GeY23Ez+NzM556UVuBuJL+Z8CE/GI9cz+aTfeKo5XRdXV3Yb7/9sHFzp8R/tMjc6JJPmq2TZrOktLeznNR4Jh7/5vFqTFpnC85ZUiebrB3P2oL2Lpo53Irdq7J30V6pCnkb1dPHYErbLAYF8oGrUHaICb9P6JDfox6hGiGjZBY2WmNJnBVzRfABgLm93WPX7nd+SWwQ+YYG39c2ic3dcspftF0e/64XMOpsEYORWtzz4L8QT6YwZ5cZOPob++n3xLWmNIYrfnUhbjLIlBAADodt7s3hkksu0ech4uGLWy5yLh4iRdYrcQuQMGioRpuA6AtTVdU64ZCmrBggdNoXijpF9f6yTOcaYCFu3U35UFGRzUVarZOGCFqjTRgc7Ed35wYM9nUpoPAeCo3j2nP0Dp92qRpzo3VUKWusiyIYsAAoGNQJUAWWLnqzIkacKzD5YSJSOw2aD6L7oCpIHb7rdy9Zid5bh5vERyg5/7pxKFObYuFkCA6LPF9M8r9XrF6Jgw8+WLsxHDI0weeAXPgsXGSfItlhm/lUfuogQqUwLvL63FxDrsK2Le3RrmYVz1EpFxm54UTU2gbvFlHM82Uc51u+lQ7REaadM+iLVFpuMPkpOZFLFlT8/Lw+GXqxgHZzmTqNuLGcmZiCStCoDqFQRH+X65sbVbMGFq1C/IS7wXN6Tm6xU9Pwr/98Q/Oi879zCCZPGKPra6ivk0S1IVcGJvj0wQrZCFZt2oL3PlqOxx97TMZnDGj+5CE6wufFRc7hC78xeb/4PT4HfpaWRoOZfR1lGjJW9PNzEj7ma3rZ6oaGOrteqiZ4141iQcQsiihtXL0auVQC6dSIUKatNAZzmbZT2ESL/HOtToxRuNRZUsrq0MG/ytdXLH6nwl3JD8bF7qOeuAjsTolfbR7wamZks9WFzQtuaW4W6M9/FzDvihceXb7SZqrh+Q28mdzF/qhj57C3rxezdpqFgaFB7LzLLghS09u1031B6iExFi/M6zgCpkKYEB4LI4cIidfuZg2NsG/pDQMzX4unCnNJU4i1NIsnhQpON3zB/F8b0pEJ7Pgz1SqOuPEvVrMQF6cDHjd4BHWKWIbMbDXCsiiqTS5yGKfuawQh+hqn2lhxkZA5K7F03m8uFp6qUv9yfB7qzPD+jWTKePyl9zGQSOLK876vMUVuPKEWgYCUqah+5XsFGu7Va5bwxqL1WLdpLQq5UXz87ruoRCifwXtgKV0ul9Ga4GYWf585vUPhGFhkne644GQn2sS8cYL4fS52Dmvw/nqdFcKESl8ZrOhiURcB1ds2rVyGro1r1eq3miLgjMycuKuMkE1BTTY3zmtVi16FZhnNkhm0k1qGwU4CWuUoO54qxvKEeizd4DFhqIbBc0wVKErPRdPeNhbxWExkHh43fuJH2K1DVVgc+gVu3TPrZHJnkhnX29uLMW1tiiD9fX06ish3Jvlm9uxdJVtBHoPNBnpHBZMslkWhsOOScbJ9O54Lm24GfMDUygtb04c3XItJNi5OeLRo42322iYRx1zXaAYcuLb8z980SwaJufJEsA6tNqE3uOKJx5RItFGKC5krh+BUeqBySoZIgE44I2px0fL1qn0AZ2VjHVKeRJbPKz10ilN+4/M+Mo3b0BPH6+8vQTwRw3WXnLZV5JM0g4JHRJjHmy2KpVRlbOoZxivvL5YeInnvv7vqCnz9m0c7IpqlV8PD5gfE3JyfMZGIm8ObdFtszpPBwX9+5d4MME4OgvfBK1nZprBOsuJEMIAZU7ZDLhPH6iVLsH71St0fUand85RLBdNbd2opVXVT/lU4U3RpdjdDqA0592bm4IQzpWJglO3AGy89Xpk+fTpWrVqlF50wYaLyVxGlHGmpWMgLA9f0DqMmAiJUyY/FLQaf40pGIBqRWDwLy1hsWMR2/p4WaamgSM7uakd7B4YG7GbygVKOgi3/yVOn6eaNmzDRLQorTNRMIqFp+Qpsv8MM+526ekM/nGybbrbT8ebxyiFlPhRi51sLSm6GrQ0wX6QwXbGc2vJRLSrHAecDshzSDfG62sAmmmxBexFU5b91nDu162LUl3SCxu62Gh6omaTcnxvAvu9zb3LdfQ3hO9Kim6qYNTPcV99fjOXrejGaT+GC074rSqo8Skm/lUAoj3zr9mpxVSq6vuff+BgrNm8RtDh3tx1x+P5744gjv4/mtjbRF0zuLy+qgHoOmYwUvrg++P66LvZFpFPDAXBrADF6MnBxU7PA5PcZNI1qTFFZQ6pmzdoevZ2d+OTDt5EcpuItTwoLZnp9l8owyFmt5ly71XQ05qY/aqmgNnZsCypl159xs5+e88TXDHStXSwI0SKvNV5MgIdQnkVEcQ1AYlYakyZMVNQn2iI1XOriOWRF8JaTmBDvOUCdRB5RbvAgGFBxwEjOn+VCb2wwTRfeQKY9zKfItDvowIPQO9AvtMEKSFOy4kPke5Nv0drSqmOTn5lIEFEOiY9yBpHv75wUfERmFLUGi2HD/BLLMko6MfN+m4DhZ2cdwdcl004R3M0OMiXQguGipH+7ok/JcHPVE9b8MTYfVaLMCUEYsNOt4Wvr5rsHqCPVTUfx+2aOZdLN/iGzFmE3l6/pU5e7HnoRg/Es9t51Bo44ZA9ZPpLiykUqgUxdX8H1B6BBkUSmjKdffU8qAMSmf372KQhWysiXR7Hg5HNEGFKgcPdGRL3RUd1X4vg+hVIN4VTUmHuTg+6LdQY0gRJMs4gkuSYZZw9m77IzNn75MZZ/uRTDQwNuiMQoFIIcCy4tVJS20cdqNOdYpfNWFboSHMXkcR0I1yh0VDk0ntrMAOQW+ecVLmjSV7u6thgRRlLO1K621rTfmXyQ4zo6qumFrAcjpkTa091tm8ulEuIXSFZsFB0d7diwYb3lpoQF6+sQGxxWpGcRwyjBiOxTDHYcecNWrVyL3XbfXdGnne/rFG0ZFQz6MqTCR/GIRtrIJ7dpEU4oeX6KR2b4GWwkzaA5fvFh8bMwQko70A1/cPMxv/dEtWpObnFEx6/SOtfUIaZuC5xpiEUtnQacpAyFMDw0jLa2MWqu8elq0typ0+rEcEeznWzW3RUW7FAf++wG8/J1b3/oJSRGsrhq4Rmo5C0QqSaqGgaHNMGlIoz5MgJ4+uWPsKm3R+nOvrvtgEP33cOYlnrPGiw441xjO4ZCVlS6Ti3HIsnNicdjxrQMBKrMQk9RVuvdMVp5X5i2+Q44f37f/eZh3Zcfo3v9KnR390gn3kYafXeVFpje5nYrDOzxfk44aJE7Z+5wJIhpkycgMFqQ1qZkSdyAuq9lBKNuXPmJG3+zdj4nQDS6JUkv9zDd+BqbGdyxGqgoFbFq5Uoxx3gTuZt9ZOToHBcmOTBaXDW8IWSHGSd6YHAALc2NGBoeVg4n598aE/ThB2UzSYsgHBJph1G9f2AQO+2441YHXnW5LA/nTeJRSYzVICtXpLmcmemCR0l8c4Q3jpMoflEaXGcQJcljvsPIPxmN+ftEk0xZ1qp7Ug2Y9nAjcMN4CNK38n0TSAVZBeraeRKYbTDr9vpFY2Qna1D5CM6GCL881YJ/D1EiryaAG+98AolcHtdd9EPj9ZDsJSYnmY5GRxaxTfckKibibQ++gGQ2g0CxgEvPP0U/Y1wUg/oaWsfjW9890bq9TgpEk2MOReFpGwlbv4RAA09znWxVEwYeuqaFbleKrQAAIABJREFU7um3mUIB++21B9avWoaVX3wiqRNuSNlWeoFXFxB0gjnBV4/hu5giT1IfyTmpP33aZARG2ccw5IrL1T5f2DrOHu4d2rKyQoomYRzyexVtXfNB3TweRemRanGmwsyJ1lin1ApBAfnlstAW/jwjBVMDIxTxoW2VemPEHNPWogK2rXWMFjud1QihsStKfQ56w8QTcZ0iW7Zs0bF73HHHIZZMCDXwVFCPSavx4KK7eVD7DWo5HTnMvhfgF7qnMnhsWqkCh4w56e1QGR/VGbUNFeIghokvMXVR1OV8o7wYoCkbDeuKy2EDzowmnHrxD41pEe81szDx6KWgayemv7/+M3HAl9/zXUV7yAEpXv3x/qeRHEnihkvP0ubRCJ4zD+Z7G5NzqxrYR5+vxH8+Wy4EZd89ZuKoww5yHW0rIP0Qxde/dRymz9y5unD5/mzfe2CCdAYO2jAYaEibdYKABfYJmkz7JGCUCvJrOPw+tGUd1i5bjM6NGyQapVOuWmQaDcCcNGyRKyq7ItxveEpr+7/X1UcweSJdnw0g8WneSy++hG8f+e3qqaYmY8/GLypijVE5NUSV2oTSD36PBYuGF5zln0FRxiNn1Nhu6nZSlFIu5nYSdz01+lhdc0KEu4mbxfJhw7j5YNvaWpSTc3KHBczg0JB0ERm9OQiRSCbEabBBBeNFMKrvudueeuC77rG7Lti7RFseaQvaD7radDkbOSVh6SLts/4Q4cFkxiyPJGJgHG/Db014lBuTKZBFZmuYiakZNSy4xIJS72mRmj49fqP4op1Rmr9DWQd+2cnh7Goq0KauBgnCmCK88T555MU8USlGb5GagWUU6VIYt/3lUbTUhbDw3AXVlJIomGqXoNUDPP6FqlTK+PNjL8vNgr6l1/7qPASDNhDMk0mwndr6Ja2B7//4XJQrtUKVvLjmQL/5bVK2bSQRA+cqeeTKiobOedGohjz0vINMPQKYuf1OyA4PY83SD7Fx40YnYGVQpg2X8ICxAOkRGn8yKBd3C15BlHWUc9ebMmUSRisFBFwur0YZYWQKqRLoYFAtuDlQLnJGcj3MfF6teEYH5qjSPXEjcSLWKOqYczMfMn+GI2z84tHPSKBCTJ0//pvRO/m7auNyAiVrtE0PJ3GhcbGT7MNCyBCGAlpa2CBI2s1X966gaELJsP+89RYuv/JKFWJMAZTLbjOLqVa5OqU2zqYbRENZFpYu9fJdTuW8VW1rJw/tbrra7jSnUkQxYpqc1NykDukLaoWX6CAXlIMDr59R2r8uvVG5wb2XqUVq6yJaGmIQZ5I0VNf1NajPHLFNcJSLvE6nhRh2gRos/moDnnr5HXzniAOx89SxQqY8NZf3i64RunZFxhqkcwXc9rdnFXEPnbc7Dtlvjnj+vEde60bNM++wHIjg8CNPEH/ETjxSKsqia1DGL5kYlqMyn7t6KWxaEcWKRHQy9/X244DDvoGWpihWfPw+1q1dqbxZ1GOHWinKVKzT6otLWxtuilwcFCv69YwE5ZUxc8Z2kqGjrQwZWgZ3GzLFe8gJohJTwYIhYoG1X75fIQpBbWy+J3NyLjAhHnoBI27xi+kHdwsbQuJ40BsoVCNuMNONwYEBcU1axzRLWH7SxAno7OyqylnwgXGuj5uBBYz58uT1gK2goJ1JGPHEsJoElJEmvso/x48brwtdv3a9CldG/v323Q8bNm2UZIbx2M0B2XyajCAm2Tspy1qE9jeRyIjQDi1ia1D4LupWixLeKD/44PjhUvUye3Zqv1hjyuHfnFvNZBAbHnZNJsqbmTWjInF1ONvuazXXdJ9LRzy7hT7qq5AKKJX0s7EiSyGIR55+BUvWdOGSc07GmDqTZ9CmCQRch5E2hmYLQ07SY0+/iJVbUpTExW9+eS6C5SxID+C/M4Iz+npSl/JrAHWtEzF3v4ORZ47PAjQ1ovu4ZeNG5DJJxAf7tIiGYzGlmPzsnL4v5AqonzARRx91DBa//xa2dG6U0xx1L/1ooBa1BKcsgvM9pRrgUphqurlN8U4HwJnbT0dTA6/LMVhFKjQilu/s0samQi/VGqsXAqu++I+2DZWWuLCJf6sACwRF8Bd9kuSbsHVF2V6XUhVHnKK0gTaIkTk0ix9SNg2C400LSauDFzFp0iQdV/X1tYKv/IX5zqj5C5XROmYM1qxaqVNFgwluV/Ok4YnT2tKifI353kB/v957n332xfTp05AjIoGKNAb5edQ0crWAF5nkgrNc1XNDyjYYK26EczN26q3K4au4tpGVchnORFqzgT5HvD5GZbXyS9YcE+FrtKJTRqmPclQW3TXaoEJUXITSyecGti233Cr0xOfC6XXDxf34XRE1FeAP9/0Tm3oGccuV56vwpcYkPwclJnjNRML4FaUlSWMzbr7778jky/K3/+aBeyklkltsVeOQqZItds1ThiIoVCrYdbd50inkZxiJD8lGJx4bQCmfQV/PFpeeOZFW6pjni9jc2Y0rfnM9Pl/0ITasXVkdKBevZpuikvfcBx2/HrY9VQWrOpQmWDOKHXacaWmlWQ/p9CbXitfgg5GN7bgT1qV8gXXL3pN0c5BE9+SIQHu/q3lUc2ZTuZ1DEDwJKZVIWn5b8Q0CqNo2SV3jmLDoMNqppThUxiWiwEYRdcGZprARtWH9eoO5XN7rtTS4q7mxpk2fhk3rN2pxjm1rU5OC/6bFWlODpUuX4oQTTkByJIXtd9hBRSGbObIrFP5skJ3NJ5ogvWZKSyRucTjbWSu604C/4/NCLlyxHl0Xt+I870k15aCxUpqSwYVU6NKJxC5xxIhIYsxpgNdSGS5AmbQ63XXee+lPOskKQ0QcehMISIfEw3JWTBZRWxPEr2+5HyO5Ai4/9/toaGjWfbAg5KjJHneuBLFmfSf++fL7qBkt4+qFP9YRr8UkvlBIea/nJYlIpf82G8NKIIKDDzkMQ4NxlAtpDPX3oS4axkDPFsQTZqXOYKN7G6zBpu4tmNDagb3n7YNNG9Zr5pKgga1KI8/pr+4eGxBs/Jrql2Mu8lnx/k2fMVlpiigCCkZbCXSia0glwKBk1j6+M0yWpuQrln/2hghapGgybeFNrqurVUHI/EZFm8OUycuojZhzFzW5iSRQ95AfnHChAfTB6kQNr4c3c/yE8doAfE0+eEYRcy4wCQw2hFhoUtTTTxt56irzblXwnDEk3dfNczJ6efiPBS7TkpWrVuGwww7DdjNnbG1juwfqh4oZBZSe6DXJxbGF4Qn+6qq6yG6Wh3YaFKWzmEchn3GtfagTqEXpoC1RCMIho5Jy6FsYug108EhVC5wX6b7C0WhVVsKKXQ6ZUCuGzTlbCFzwdsK2OEjQ3O+uuPk+NEXD+MnJ7HTaZJaaQCoMmX5xUIMO26O47cGnkUikcdQ35uHgfffSaczPxvdTEJIalY268X2NNuEL3xDWrVuHY445Bsl4TIM0lWJRuTm/KIXnkRk+W/7swQcfZP8Wi8uszMSLDIlS9K64lv02fqkqzpWbB7FizQas3NSJeDqHMxcchdnbT7ac3XbH1r2wDVnLj0Nq7pgFvAZU3CT/+q/elzGABNGYtKuzxtzLIhzb+aTO9vcPiFtSXx9FX28f2trahWw0NzdqCELcg2JBTRu7+Djq6xtVqU+eNEncFObbdioE1aHs7aUhasqiHfOzckE5LuvukRTnAe2Gc4Ewr1RzwikyMdprvIq880IRU6ZMwfDgkLD7gw49RIVnx7hx4l17gpIeasSIRbzXHvlgOsHFICivyo/wMnTWSKGqLAcKRkvUGbQIpiDAuU3XCeTJRHiTUZ6fu6W5pSr0yS6thg04OeO44iT68+dYx/hC1MOFagY5w1yNoVUqKvJ439ijuPOhf2Jc2xjsMWsaxra3V+dfPd+FfQ7e15FMEb/90/2yr7n8krMlMR1ATXV6Su9HeTUuMnnUc1C4RvMCEydOdB1gOx3o1KZ5WKJxgaB44x4tY6qzfPlyHHDggfqeBiDYH2AK5kyCfU3ERe4n+5uaGqRVaY3BID5evATPvP6RisZsPoUfHHk45u05XYtbHqvitGzjXeT4VVUxK7eR1MDLWT0V2LTyY9mO+2kfcsljQ4OaycymR9RW7+213IsRnQuNRWFyhBi2Da/yi5ujualJF86fYT7KHU7RIlbaHjYT/FiBSPV8aEkqORWLKq5oj80pf/4b83lyK/i5hoaH7Ca4gVjCbISIrAA2o11ClqW8WU1zJ3PBsVjddc6uVuAEyA3horSWv1E3baHzukQn4MNzmL9PV6pUW89hKeUwPNiv/DvsHBeYwtk0DSO/MeUi9axXqOhVo/SEn5EL0E+zC6v3cD5nEVnoUbrOQWks9vjzngjFnFyf1TH8xNHO5XVvaHlYzWndNBQFmsI1ATz3ykdYvGo9vnngXBw4dxf3eraZqaHO52qDKUHdM5+q8r08f8k3eoZSOTz57MtoCAex8/Sp2Hn7mRIKooHCyEhWpl6EEfk6PPX8iUBHPDajorUmEyfNw8ZGg1+d0zbTI270Ves24r7H/1ebg32TQw+ch+99c669Fkzck2mW7+76NIeGuls1dqzG4pfSrzVL3qswWnsykCQeaoIYGhyUKtLuu++BoaEBdSn5JHy6wYevvJfcDB7DIWvadHR06Fhh5JJgp5wXQk7ay+Ghkuqt16JjU2jDhg2YNHGioKkNGzcKZWG0b2po0JHHCySawx3fublTr0mOBiM1K3r50TMiRmp1ckjpCXas77333joteMLoCHYyxORI8LpV2JBA5EbtNJOaNdqxWuHu53nDNDRSpnd9AtnsiE4cy/ntJKBEhKZweM3SewlIUN+/h1AsYdH289WZUBn1mg0iPyPvKR+RDT/YQmeTxCMISnkqUBHLApvvz9fUCJsTexKnu1jC7Q8/L3OCheeeguYGk7AjfKp0VMZmBAgiqiH8e/sGld/wRtgq4qXX38Pazb3SqYnHkrjh6oVoaCBpLKAUhg0iIXC0CK83LrmCBQdLMjTCNVjTFMEooR1EhPooVem7ADKFMq66+V6leQxic3bZEeeccmR183NdcL7TD04wg7AmGi2BzFfWL3D+t1KgVV+8XRHpxg0RcKexQSFs201xixstO4uIEWmCPKqSQjpEaRQ2bvYpjM5KQUIhTJk61WQU2BSipUgDlXDLTrUpoLyVcCV/j+nG6hUrEWczqjaCPffaE++8/Ta22247DUETeuTCoKYhPxsZkGodu+FmG/YIK1Vgjt46xlAJE/vJY8eddkLbmDaURPc0X1BN9MsnyTqcfgBaMKlwfZM18DdUqEo+i8GBPjQ11iOfSamo9YhIvlhGe0f7Vgc5Z0/joUpufOnQCIYsyOpEtFHWIrIqlICLPXSHV0uIlMHFDSJ4mFOzi87lONoQrYowWT7PDm8RW7r78McHnsQ+u83CPrOmIlJLz/pGpTaK0s5ISt72TnhTC1+KB4Z/+yKYfz767GsYjKWEoPHz33LdpXKkszTZUi8jusHl+NajCLoBb9KUbULIcmVrIlqKTZTNrjuEy2/4i66BG2PihA5cu/DHsnlkjinBWTE2TU+nWg+5+2QnpZsHduOHgWWL/l1Rw8XhtnxzphrMywb7+/TGbWNaRGjfdipDrfJcHk3NDVocjKBs1jAn5a6X/qDr9vHCmMow4vImEwrkvxFtIVLCi6VEWOemzbrg9jGt6Ovv0w2ODcecYkAZU6dMtbZ+Y6M2CtOA1EgSiVjCiGW1Ef3M2nVr7MRhdCY8msno882bN094fg3hUDd/KA46WXNhavKZYqyPLHz/AocdnMiPupkl5q9GRe7t2uAMoazjW0+7PueEJ843I4t7eEo7XDDhScH74KkGfsSL127Qpp+7ZB8iYixCR332hDT9jGKP920aVYrJ4MLPKWXaSB3e//gz1IcDqAvT7pvCmmHpw4hPXx21s06xilANQzAHp9Q1ZZMtAPAZ/v3p1xFPJtDdtYUSS7jzhkurplweVSLtmKcgUxRfbHpOjzj1DCbsWbiFyHlintLGoqZ4UgG/vf1xXXMqk1Gaevs1P9XJRkKbBZWtdGX+nffTim3j1HDT+oEUyeB99v6LGprgN5kr8QMysvLPkURcC5Y2Hfw3LkYz0LKWMXOwzZ2bqkQn5mK8KYw+pjVu0/K8Qb7oEFkoGq02TPzPcXNEIxEMDhKLtQ+t+OBkkD1yUHTcGS4SPmDqhdTAkBcxC0tFsMs4ODhgC9xNp/Df+BkoQ0b/nmkzZ0qEk69BZwblyJTYUB5tE//WhbMZTx65emiaQzW222BPp9rSHePHKX9kJFaBpql8N5jhNF18p1WRzU3783UkuuRYj9pErhFUhRFFdnCQmXOm5nvIWcEJgDEF80c0768GxENBpDM51JGspkGGPIb6+qu8d0ZKGk8xvTBSmJkQsxi2Dq8RxbguPH3ir4++gsJoFv29A5g+Yxp+etr3qymJ7yb7mVaeCOqmcqLfbVrPHaJ1usfLCSSoCcbCXJNTAVx58wN6jlzkDEJ3/PZiTeITpZH3kCPm8T7onrkusrhCXofHDbXoxPv0nWcrHDrmMWPcZytwOjs7lTbwF9UciBiHQzJlxRKaWxqr8gpaYMGg8l4q3DIX5KJlOuM1x7UYyfFWzmZQITcEc2rPTWE+6QeobVEWFaFj8bjGwaRBEg4be9GZWhn8Z/ATM3Fj9xke7jtg3HyUjeDD5DV89dVXOPzwwzF58mTLGd1IGBemcVgMfVCjxEmd+QilFMNpsvC1rOp3Y2quPa374WiyGaZkzeYV6jFwNi7sgLcOrWz+QsbT8TRSO4rdwAAhSD4sF3l9rsuoyLTKNrdpuvjNyufBZ8DFKjTCj/Kxh5AaUfeSxDIb5g6LFsC1yN8xrhGlmu304f1458PF+HTpKqFejOYnHXs09txthyoi5YtMPg8VyNt8Vo/aVT+3S2994LNNZg0cpiJX3HAXiuWKFjnvx23XnKc1w0ESnbSuG6TvOcEkQc8KFtblNoDDvhdY+dnragZxITO0s4FDbnmKw6QUR3ewn+cbcBGRZ0KhRmpwcAFxMTHSU76CN2lwYLD64L3vO4vG/oF+0GuTd9MPWvDndaMpH/b/VHXmwXWW1xk/V4uRF1mWheVVYGMMGBzbCekESIb81TTT/9oO06YzZCZMOw2ZNjDMsJSAMWb3AqQsTaGlLQ1QlqZpO810OhlCmgRIYzazVMbGFrblRZIly7b2rfN7nvfcKy7DSLKuvvst73uW5zznOfPdbUSzMN+PjKI77iri0uUrnVhpqrLxVC7QRadRHZPueS6K0AQ2nLnkJp7R9YPnYfPymZ92dcWmz23U+9tXrrBkWdSJUsq/4clwo2PD9iqy6DQST9hjcM9I2rKLPNEYLzSXxbXhYBeWknve9Fzk1i6xIWETAA/mwjbdwIuc/6hjOIZ1N35KcPAzf2/i2WdJYL4/TdYSLPop2mhlYyLuoxGPTL8TL8li/MTj1DKYlExyTdr73Cv/Hcd7elXCHx0fi0fv3xL1M+POrwoPnnuQfKHkDOXCznAo/93FLyMgMhYzhHvz1SN7xz27YnCEgp6bpJ/ecYvgaU2HlkCU6QgilhXUPGdAkc9neBXRoD6Hyp7XfzwjZGEWJ9hDZU2H5Kaky8JFpuXUDimIg+K8+fPFYSGOExRXuks4BrE3cTgXzCLghAgLzPm1y+FC+Rwy6qXtS5QDgK4krIcbymQl1XFZ3DxYJhhoMnMRQGprXazuI8thmB6gxmyNVfHCEZdlfDzefeddYbsca/36y2JipswvZeKcqlMlsZo2WnP27GktGjxMFkzofk+rlPFiFlxYhOKJq4PfYUdO4JCQTtF65N8NOVoaO0M+9ZYmz33W2MGsiOSiyWQLQlV6sWpyF25ETyya0fAqrQilce8pjSYyFhmWFZQC2jHv+8Gz/6E4n+om57j97pvVUZQWHPhXa0IirfWRhS4bObcBZo6WkHPWJXIzay1AWXjkiTh8cqhM5quPR++9WUYDXRWFaikPUgpMRB8yLCAvkrVzhxYOk+l8lbf/5xWRu/igrGyqIFRguRSwZPESqvDKClt2bMAzATZT5iy3QhuTNwS0XS6Ov2HhcWyOlUw9/lZWplTf3nj99bj885u9YZrmajFRRQQJwDrzIPAaeBCSVYZ0EduSK7S1LZa668KS3Fp9IM8ZPXLj4HwW/O55TU1xYP8n8g6bNm2O40ePxiUbWOgmNUnGbaroweSUB9DaUlXTuSkhdHufNnGR9kiLzCLKvELWvlQw3RHjBnLumZCdUoziZ2Pqpk1YWsNeS265hCW5aeTFSrOFaLhDQzou9zk3XQqFskGzesriNbzphFtyGYiXjsK1MZJBRkhB6R9f/okSPEh4rNuHtt4UUxM2gDJ8WkMswkJeEwOUsjz33VylfK8TbMOLfM0WQa2nSsRPf/qr+NF/vaYiFffzBzvv8oTKVGgguRdEbM/u4pADwCz+6Z6PTkbXke6o7P7ZP89wkZ6+5gVA82ouaGLGHFzEDnbVcI4QGHZ14us5kxKLBQ6ayassVOMc03CVJEwKShwqLVwsFJqosfSrVq6wFFoRmOzr6RPMCIzIeDtx3Avcl4kkMTTJCgkO1AJdrFRgCU8WRnf3UVn0tB6cP3/Lw/PAXSvPsqBOD56ODZ/bEC2LFsWCZivOSmS/yEKkXILiXoUJ7iGkYJb02ZziLMtu92jR/dKvyCblGrNEzf1SbE5lUPqB5h1kKMQ1Oc9Ag6U2hykrfHkukmaWYkKD56sWFTKuO/kshIIYCCFBc+dFE+FRCYcSUVIxTaV3yzqQF+0/2BMv/ftPYmzEs4Ku++YfxYaLVgoRcd6jAYx6tpIuYdOgWCBZiHrNlXJoYoIWz0A5TxrXUoBT5bsuon/gbNz1wGNCSjifJx7dFvQ9aaw4z4KkW7wHIyoACRAGQWZmoB8WQgybRKoFb736groHCC9SVyPxzjwpY5vg5OcoTtMg14lJUToRy1S1bt5cxdM8JP4+kxd26eDAgGSCp2bsnq3z7YWSN5cQ5P86P1I83XO0W6zFpe3Ljfg0MRTJkGN/PxOGRxxDzCD53CRsnB1N4giycvrUoKwYMCKJLxY/4z9RY7WhQ/E5MCMblhtPiLR+/XqhP5w/1V+42ywEDXUt1ci0QFyLQqZSNbTsg0lU1nOUDpoeJm4b+C/du4bkFq69O2JgOLqCC89ntu4h1+pOIocXWYLPkNDimqbm4UEV9pReyVrV1L+vJmOK642sAMUKGZLl9tgYbq9gz0ol/uaZF6LryHFVswEKHn5gS8xMDet39jZUb2sCrgAEpu26YaO5xYk3LESe9+zFnd9zXhlezdTXx6137pTiAIv80V1bojI+UlVmEA1DOvXZ4kcYaI8yOuLCmNZD0V+pvPPzl2byJvFVY+OgLxb3k2L0xm/p5JhxkllE1MEuXVypq1os8639kivhQpubq+gM/4blt2inJ05Y9dU7HJ4IbpUKGq9MlvAGxJXcaLMiJ9UYTPEKV0iyjFU91d+vC2ahc8PFNy7KWJwrx6HETN8p17vhssvi0OHDVaTngz3vx1e/erWKOqvOO1/nRLKWMnbVhLAcM0MCFqHkz0rcqM0kuQnTaTMxTFddRYY01cEsvnzQhHFqTClQqe4DdAXOOakHZTyN4vwc2Z73fKZSUwcunsrQoJEgQZRlkhzGh81l/rlx+lyQFAIf2PF4DA6PR39/r3638/7bo6ECnbcofvHZRd0rDZeNF3ygBlEwDG02V9dEGoqMy+2tyNPrYnxqKm7b+nCMjLra+1cPb425mofmvIu4Pwt0OWGPMZXwlQR7Flr44Olh99S+8/MXZxSolxjaWWtttLM1P8w85Hu4KHxYjxokmkQh9cOqc9c9zcGlKgocxK7COi9saVHVkpiN+THwn4WtFjgJS0SDLNZEIZFm3PvYyUV3ccGNsmi5pLX2DbNEAnDomcFB3RxDSoYzz21fEv39A7Jv5AYUhVhE7nCa59L59LQWEcelUYMF1t7GOU/EuvWX2pKDW3OzC1E/3b0LRabSWh+lZjUzuc6NzzXlQiNhBsmwJXPLnYoyRcNRxY7RUSEPSYeFuZmQJJ5IECKsTklK27NosWlorgccYBQIiRyi1RiOysXg/zfMMUe+kZxpfpVchX7o1vt2xvjYZPQOnowLV18QN337WqNAkynGRJXVFWPoyzw7y5G4jG+Dad1ynl8TsnRFWsKMUHt/v9Gjzm+5e1cMFav88PZt0doEz8U5RCb8ivM12sXdU1yLKBPlntU1oP9zJipv/ewFjTjMcqgUQgt3mgeKBWJxEjNjXQg/hJVrRj2EIVcIscy4ebulUlAoo8bTgvA+mHxk6aAAiKtz0fAvcEFoCer7PIbGklCidhJrq251VIoOiYn7BrkQwwLp7+vTwiBR1eBZbozE488RuR5PBceG8Aa5DD63C+pA6+Lo7euLwVOn3Fg9MhIDJ/tj7dq1ml2D16hvrE2rEAU3Z3MmPVfum0wfT+LpGYQiiVZleFYN2zQg1kUTy+lxrZ60Nhvrz0LKbEQCCoSQIhVJSrhSULHahirMSgxP0SDMc8lQwaO8/XlqpAB21XABOELjcec9O/S8zpwZjO9e/2ex/sKV3lRSIDOsR+xuL+RFC2SbCFQqh1XDU62xVAarVZidK5EHTcet2x6OM8Nw/idi+31borUJDnDhkxeuiwzDxLSluOtNGebvZbzG0HKclLGqvP2aFzkxDDuNrywaMleosm58cGkX3oUUnvR7XFWjUA8sF4ufjcCrHWWskyerrpedlbFoTtJN7ZBsQGVxJ3WTG6CZnSUEwTojW5bFnEQOUonL1qBOYdSJE8ej90SP0BJweQvkz9F0B8IUeBfE9nT0yBOhKVimIjTOcbFhUVEuUJII4aqxMboPH46WlkXx+S9e7nBBnGsTwbg35CjwKDLJ81x6L8DE1Vk83F/NwCxTJKR5s8CPOYewAAARqUlEQVT6M9wjy+5VlISmS+eYRhC8WTRFujQb8B2eMi0h15sKvLaQjlV5kaBhmKhYpyGycle2oFlGD8+HeD9Mj7ff74x/+dF/xmnYhmNT8bdP7oyZyXEZKnoLVM1mo6JdoM1tZCgT0BK0VsM1hUllkXLOuekTppZBrGuIh3Y9Hod67bHu/97N0dqKd7AXVbRR1hTXJ1kSkmC04AsSxc/0Oxzr6cOSP6+yfsKCTjJ9Cz1hzRRGfV8SKFwihRVZUjU2G+pRIaivTzuckIWL0Fjpc0BXEH8ELoJvciYWt7VpUyRKIRdepjhk8pX6JuJSTNVUvji7lAvDWkiOoTQOiG45YVEhHjifQ3iSY2C4VjYt1pxFi8afj2cxHNUMuNENDXHi+PHqAiUE+vjjffG1r/9OLG5tlZbj1AxkpqJgq9Co5sUyVMoFTm7AvyGyxCACPWyJBRHv1z4/DYwhuVoyVvO2bhSXJRTb0iAOz408KQtFHEe48bjDCLfceTE7BGWxwxBNnfGiXlDx9TAArLFhbjz7/MvxUefB6D9zSoKmj++8R51FvKTZXgaVEe7yIajwZjiUi7hWbCgCQAU+/UzYVDaxWx4r8dyL/xpvvveJwqvbb7w+2lqZ3OxOoXzpGqHoqu3LnzspLsuYimdDIxNigcqS58nY9eYIQHOuiRfBTan+Yf3ci2kp3WpSqrEkxit5yYWpSINmiLvOQQzEsmPzaHDUqBsAMikqXdz8fYoDpVtlIacKbMJPeoCSiLA10AhBBEeLbjp/A5bOi+/RCFFvqgRDK5akK5CcLKVK+G5MGB4+K+vODWWYkxLtIUst4EpBYI4dOxbrN1xm0pWaTuC1JL7tEMWS04WzLuKXawjZIpg8DFl44K8yaItcBbK5mnzL6JVsfK55CrPw8CjJ++b6OU9tWFnJWsijzVYQLYd9bqY2EpMol+nEeq+8xlQ8/PgzcbJ/QEjal6/8QnzrG3+oiIbzoDosSHDC4aQaT6pjJXmTNzLX0VgEn/iZZ6EcqIAKuf4c7hhQeG/PR/HDf3tVIfKN138rLl7drk4fRxqO4eWhyoAuN8Eg/WFNd3pNT4+Mx6uv/TIqe375smF0Nfz6w7lIYlIYgrg2YnMLyLuVi1finQk3EjrQCgUGjoWmCKTBUhMTRkpOnapiz6IMSHfD1gpMmvCGYg7JYVoqFhUPIXkIvJfBprzHHgBejUdWszl5wDmZwe6Pm1JGrpTN5CR6TixdtizeePNNdb+w+NkIlLatqmWvgWUcHXIDCNeEQsC6C9bqHlGs4m/XrFktWNUu2A8/q59GjJwoJY0XaEDDtKRQllIapXxfprw5kbc3TXpAWv4sOiWakjlBHi/DnkEpobnCmkUYQss8Tm1GlIf5ikiFBy5a71hNznvb9sdjYAD+/Ej89WM7onF6PMbFxDRKI4FR6bx4XSD/jEG0qlVJcAtPR1QInkthEqYHzXOqJsyVSnR1HYpdf/eiPPCffvMbcfmlqxV6sejF0ymficy3jaeFSIF6LXMxHYPDY4rrK2+/9rxUd1w6dmiCpUmcm39nB2Exsr2O92X5XoSuQhDSDJgyuQ1LRuKHRcRiLF+2XDrkubiN61oISN3WBetVowEioqV6OFsAKHkeziGcoPH3wIrgyNxAHgYJH6EIirqESRCxMCpUR9k0eIXWNsZZL1DY1dV1UMdYtLBF8a00xieAzPoVErQvXRpHu7v1u46Vq/TeAwc+0QhyEtuVHR2xdMVyyUfkK2NNhy01TUa/x8iH5OeqtFrHmbWma4d72RGaoYs9pammjtVdNc35qpncJb1V6EL2sBbrp0nWiDiV2UZO2k0fADwwAS2ka3PvjifVIM7n3bvllmg+pzHmIglRpODwRtx3WfOoqPEl0ZL8Oi0hJ0OT+grxq/B/8loyzq6ibXV1cdPdO7XIf+93vx5fu/qLWsgaNlYMnBA0eT8MZgEf4P9PCSiLgTMj0TtwOiofvP7KTHaL+wHNxOLFbbKscDLMObB7kGyzhriWsSbSOTQMSKwN0zB16TiZRa2LdBy42rzPsbN5JlhOD0pltMb8Iq/22XiLG6AumUK0MkznRS32orgfdOzbimYIk7AV500CnTqHq1Z1RGdnp8INrouQg3PngSOqRIcSuuiw8xDX50EQZnFcN2SMK05n0asNK2GrsTFJaYDC0NShToLSECy8WTmK+eXkFhnCcFli/zk4rS5eJ1duqK5tGn40ZKfEtHw+Fi29GhvapXQP5sr7gLVPDUaHm6k0RjWbyqMEO5wDpIWso6H4UDz1989LmgSC3R1/+efqFVVFs/DuZQSnrRdJc4z6VznvwosHs86NR0TgxV6ToqivsxCUOp+KWKm91HTcfvfOGBofj6u/8uX4g9++qgpypCARn53sS+BCjqtZSzPc74jh0ck48OmnUXnvFy/pVma5226InYY+iWNLYi0qcE5kDNCroVR0UIP0mR2n5Bg/J086y9petHBCjJ/nBjJ640pokqyqu14uFwycVjtCl9KVXlrXCGXo3OfFA6PsXCWJ1dUL1ycZJpZjIYsnD9MReYu2Ni16qqSewGBYcv48q4UtX7Ys9u3bp2tsnjffClWNDUIWkO9YusSDwVjwXZ8cFLFs1fnnRZsGCOTyzNlD9pachx6G3mAXS/KucGaWFEZSIBSf2+fpq5ESw6X8RousnPds78F7Cc14U2LRqJ3lpuA5Z5hgUMEd+xkr82z/4bmXYs9HB7TRb7jhhtiwflXU5+DcUYd4arYWMat4MVr4JOfmn424OAlmkWfrni8K7+XYXAl84YaLdTkxEbdt3RFnR8di/cUXxXeu/f0y2IzNz3Axh3uWJZxWglnziuQYDQER7cTJ/qjs3f1jayFW4RmyZiy1yf1CXiQwhEv0AsvqFAdvaWnWourt7XPi0VCvEABXr+aVKayFS/KgHA6JZqohhrDRErbMhpT8kLzwkPk9//w1skZr1qyJT48ciS9s3qR5NyuXLxVHJRMmjXcZHpEqF7g2m4ONwDkDGZI8o96FbAQ5A8cknOns3BsdHSvEW+k6eFCV03PPbYvdu3erGMUmJx7kfHJ25dq1F8TBg10KW8Dd93XuVfvelVdcEavXrI5GkILSqZ5ldsGAhTRGb2bGzdqkEkTKwV+lQlo6+1kMmdgjLZohW7r9nI/kceew+TxQKgtI/DuTilkYqVzMprUxs7fmBf884/1tOx6LE70DUkh46rFHolIp+imFm87UOiw/BSlosaJ9lIpjts55DXkGaOZzCp9K+Jv5izhEqsi64APr9K5tD0TP6bHoWLosbvzOHwumNAxbJoEIdvU4+fROGEHicX6Gt3J2dJyKJzE5m6D2wcQzCNyDQHh3+QZjGSTQT7tYSQhNjmLhe2wISQfdOMyMobIpHRFEfDRDyFDlbPqrXarH1SX2mckvYQqhFJsIKIxjzm9eqMro4UOH4sSxo7rA9qXt1Zge+zE0MloYeK6AJR5O6OJN52YN5hQRToGtt7Whob4/Ojo61JBNzNy2uE39palnqFh/0SKNgHFDd5OKSd2Hj4ofkxDqW7t3xyUXXRybNm+OxrlWpeVhzE6wsIC5yBMDV7xeQaICCylgzAtb32eoAguRBooyMKu4f92/Mo5Elr1UktO6SQO8JII2LNagVCEpJ1EI27f0A5vk1q0PxsCZIQ1K+/79d1W1WSQnYR9URtgw2jLntRqpMXzsTi0suCICdWJVDW4tjEk9FjW7+D4RAt1x931xYmA0WubNjXvu/IuozBBJTFjOoozCYb51Mj0xEHwAuSfeh57bwaGRqLz7ixd0N61JVxcrVqyUxoqtaBn1XU6QAg3jSdKleXES+xFn18YP4kqwlBR3QCVYpFw0Av5wRJw0mZWWYQm/T0uVMRwbgsXEezhme/uS6D1+TIKfyEF82NkZF667UC1zX7riS7GkfZlCAZeTGbdXH83ooJ88WR2iJUk7uDJDwyL88LlCe6CGskEpEs2fF+vWrYvf/O9vFHcT8rB5IYYRMnF8W/wubdoTx45V6wq8F6uOyM6GSy8TD2Pt6vNiskyEZnFxr9NysiCTXelNXvRvmjg3L6VMzmyMvAAUrpTGkVoY499nl4x05Kem5FXxrk5UiyY6c0c1tcOdWWmgqt6ifk7ccNsW6Rquv/Di+O63r1V3vz2s4+wq4iM5PYcmRQJImR+LWiPJxTyke6xWzHGiaeM2+/zze57j0888G7/e0xkxNRFPPHinvAzXntZfFn/SSbgoIOIpUrtwbjcyORXHjvZE5f1fvSQ7gaVkYcj9TSEV0Rq9Pb3VCh5hCskYNz5RjoSEHMYwfqQ0HWYSMTUpHgThAjcl40CjJ97xuYixgqllbkvjjnmSTB4SoQchRV3pfiEbIKPfuHGjijSEFufMtcwF58oNGBsfVZWWG0NIsrdzr9iSoCuU99mI3d1HVDDiASxY2KwGaqqviidp5iihTooiwZZUY/ZCxm7P0waiwsomOTVgVSkWFB6M9r+VKzqi6+A+qRGs6FhVxqDXFKV4P7hwCsZn2R7dFM8vZR59rYsmjYJmVJYxirWiixd5VhTFhFT7njkx3Jts2FBoUKivfCZWXVXKMrVvz4cfx1P/9KJkJB7ZsT3mNVh8VLWCkrjizXO0etW6l7GNdD9kLybGI/+OBaq8T932OXDWtZl8pWfbu78rvv/k08pGnnzwjmrcXrXkolVYudYgBF+Z82QaJYZlGAjxgzde1syg9iXLSoKGdJgnPvBGNx64QpbV0IzZIDZZjNI4acpRQE9NTgqkLfdcEvuZUO/Yz2V2FrGLPiSl5q3wcLkZfGbKGOfDRZZX3fd9FkCiCCMJaZGWJstYFLPR+FxCFTbniuUrFHrIRdOEMcHYQFd0JSTaukiIAAkl6MvRY0cVbsGF5zqBKInz5y+wpDXYvoa84tonJ7VxwJO5R5s2bYruY0dj4+bN8cG778fhTw/EV666SuqwF62/RLDXbITDpXrHor43uN3CFiRWzxHiRbo543jLgTjurmLQs2SPEwnTSJGikQga5SG67l9NWoLi87ocRFsfP3z+lfj1B3tjcnw0Ht11b8zjmRSqbDZ5cAwMDbF4IjzVZLZYaBkLzWB1cQoPxnu4VqsJezZTehlbeDeLnx0ejc79+6Ov70xcueG8qJvT5AacOWi6+DjCzsvUa0AR4nD+5+BDFOPYysTklN2TFCVwXwqq1rX2rnJo4VjL7VnZY+mYl8FSbqL1Q8JS2dIosy7d6RwPCBFqbMb4Hi0+12623HzFc4VZlzs/3SQ/s3BBSDgnFghdPjltjmMjpZxkLaEfpSjChkV75cDBA1VOCfCVuBfEj+VawP3T++QCSeyexNXok72N6AP1DbLooDFsJCw5OimMf2lZvCTefOON6Os5Ftdcc40KbEjstZ3bJgpqJue+d6bl5n3URpguSrAimNFcXXByvX/2oCj+vWjKSL/FCT5GLcOcVO9lI+agL4UdEh1lwh+qX0aW7n/oseju6VFxb/u270WlAvhs66yQglCziDglykY4m4u0irYIEbLBURJavur5ChlxmJxl+QynZvPgxeqcmYwB1MJQ5sqYn6IaY2KE66dU91SMjE+ol3h4dFysysqHb74i7gq8kYyLU3SdpI8YlA+usRQtIJOhh8UsLR6ZDQk5Mts71ZMM8qaqAF4qgCnrlfi2iVfuneQ2Yl1YxEg+w/dgF/MzVpvw5MSJnuqxchOA1UMVxroI2io9k1hv+NJYHpX7y0wisF2sM+e/kOZn8TKca0APxoKD8+OZstLqCqzVaU/2nVR+QLLKz+DsqerFZmma2xxnhs/G8SOHhKM3L2yJVaA1DXXR3nF+1YhIqF8JamH2FTgtUa+ysqoEK89KcpHJm7iGytgoWT9F47AKdi2R/8JL53gyVoL2Epo0LQXPcdMtW6Qp/ifXXRe/tfEibahq0a4ImzLYCksqmkaZOwRfCLSlhgT52BmO6PtZn5mKBYk+JYzoIpo9m0Y3MhVD54/C2bCQLudfNLYjpGrFLtAsdQqhqDU+HQsWtsT/A30+euoe8TOmAAAAAElFTkSuQmCC">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -452,7 +455,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1036" name="AutoShape 12" descr="data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAHMAAACaCAYAAACaCHesAAAgAElEQVR4Xny9CbhtV1klOtZeu29P39w+t8lNSCCBAELABkVsS0osy6KeInZYr6TsyifvqaWWlPLQUgEFFAGBiFCChD4hICGQAAmBELpAcnNzu3NPf87u+7VWfWP8c+598H3fO3Bzzz1n77XXmvNvxz/+fwaPPPzxJBqPEYYZpFIh0pk04ihGJpNGEKSQJDGSJEEcxwjDEHFs3/P3QErv4e+DAEjiBOPxGIPhQD/jv8N0iHQ6rfeOxxEymQwCAPwPr8PP4HtTQQrD0RBJgm+7Fv+RSvFPyq7dH+havGYCu0YYphDYVRHbX7rGaDRCLpdHFEX6w/fxZ3qv7jnQz3ltfg8kGAx4D3zGCJl0Tp+ZINY1+Tr/Pj2fuwbfy9/xWnyfPUOge+P7o2iMdDqj3/F5eb9ci3w+h+FwpPfyD38fJ5GeJU7iyTMNh0OtG6/Hx+Tvdd9Bovfpi/dy/pF7En5wEPBBx8hms3pgfvFDuXn84gXz+bw2l9/bDae0CfxgLpDfNLs6r28P7L+PxhFCLWSs90VxNFkkLcY4soePI4SpEJ1uR4vAxaDQ8D55DzEXjddIhdP7jGKMozFXXBvJR+a1phtn92sCBG2avy93t5PP4D1r08OMpCIMtVa2mBIUW0zeF3/Ohebr+bNsNqON4mt6vd5E0HkvYUihNoHIZLK6D/7MC5rfTH4OFUF7kA7R6XT0GVwTL3x81iQaS4Qz2az+Di586z69izc1GPQlybyolzTeJDeUF+NGD4djp7UUAPvjN8Y0lhLETbQHp/poU5FIooajkTQkFYbo9XvaGP48HYZ6Db/44LQOlWpVCzgaDfXQXmO8gJhGcJOBMRfACQ41mRvHReB7vUDyc/nHhCInQfGbYJoJLVaAFAbDoe6JCxXHFCbTtCgyC8Xn46bx/XzveGxWgK/jz7l+3DgKFd/n19MLGteY1/LaTgXzwqJ7cGvL9ex2u5P7poBzvbhWuWxOlrTf6Upog/OPfIY6pptrNpsoFkv6BS+cTvPBzQTx96blAYIU/21mihvJ1Uz4oHFkF5XNBeKEZndkmxObKebN8zW6YSfyvGbKLSavS3NL7S/kC0iFNF92L4PBwLQtTMvcyDRFMdqdDvpDM7+FQmFitngfppncaC6WmVv+4cKbEFNYaIn8a3mfoYSMVsQ2eIS9vT23QSYQ/MMvb6LNcuWca5paI2/uKYz88hvGBaIl9CY2nU7JsvA649EY+UJ+qgjOzXHdtRfO1fHfw8EQGd1LgOCxr3064S/5Iqo0FyubyWqxuCFcTJM88wcmlXw97bxdnO9pt9v6kEw2Y9eS/6VpSCFxPk/SIHs/xohmR4tFLTYfJ42OaGJimdhSqYyApj6KpNH9fk+b5U2bTB7NEf2INp33aM/iTaEJovl50w7zX1MTTE1LT1wLBXo0oj8KTDDc8/I5wrSZSD63dyG8FwkgNTkdynzyM7S4Ad0TBcXMKv/mug2HA1mNfr8vQS0Wi+Y+5HbMQtAK2ueY3+W98774Wfwc/ozXpwL5ZwzOff0zCV9IqacU84uSzzfxDQpYnNbQLHoTUC6X9T0Xxj7IfJB3yLweF0PSaAYXiYIQ05Rer49Uhs7I3sMbl0nixg0GbkNS2iTvu3lPdp8hsllqATDqD2VyErdpFuCYb/GfxeuarzLN6HY7zu9zYTLI5bjQ9hpZIjAOSLShZuZHztxasOIDHK9p/D2fv1yu6D3jyMwv74EbR0XgtXk/3DQfbPE6fI1ZCAtmvOWQVeRmxrEsFfeE1+GXabkJFdeD19Q+Pf6NexPvcOkfer2uboQmgDdQKBTdw5qmcgVNiyyIoeSadvk/tnH0v5RGi4BdxMmgJ4owHo0wGA3R6ZqtL5dLk6iYi0JJnX6ZpPKe+LCUaEow78v7MdO8ZBIl+qjVTKAFLGZJLPKjMFm0aeaQGiItDwJpRBwlk0Ajiil4Hf3ca7zfGAVyqRSazZauwQU1y2ELzUX3wsDrU3v9z3kNaqWPgKnNuXwOSWzBlRc+c3WB9oMBVS6X0xpQ0SqViq4ZhoF8Z/DwA3cmvCg3xC8QN40PwYWgD+Xv9JoDgYxCZ4XZIZja8N9eyjLpjMyk+VdLbyj5TGe4wfSjCoLkO2kuaE5sMbkoJr1a3olV8A9Ns8XN9oFDr9uVCeai5WjiXUBkizfStfxrFS06321xggkgBc8icTO31EwJgrNYrVZDC8gvbhY/v1qtTqyXszsTzfdmkMEZN4/3YfdvQZpZQBNAajLXOpMxa9Lt9hW7+NdRiEolPi9NqykZN5TXUNqkfZA6Ifjmw3criKQqm902+xxFlnNx9xUkDEeSPMoyzRJfQ0nhzxXKO7vOIIAm0G8SAxRti+y/02gXbSLlpdD8MP94gfCmNxkz8GKQ07bXBAFqtZrMC1+TTWdkivhF/+Fz20jCZdG1N4cTbU/MfJqgJej3u1qoVquthcpm88hlzarIslDz6VLcgnvhsPs1YTSfbEGa1yqfetDaUfD5GfybAsMN81E3N4zr7PN3bphZFMutzRKaMDCu4ecyJvGxgA9Gg2889C8umjWJGY/N9zHH4sJy8xh4MGoqlopaHGqrJMIyWHudAgFz1tS+DLWOKQ6BB2eG+RC6CZfUMwCiRvPmuSg+1OfDUWCUi7lN5oNIss1QTh7U/LtpvoRKaUyofJP3Yj6Gpp7+i5I9Ai2HfG5qmhLZM9h1qJlesLK5nNNW6ZJF8AcEk5bEm28fDHIdJejOf3NT+Dw+0vfpnpl8D8IYKOBz16nb4hPbU0+sFRMImHD4VEsb+q2HPyXjyYWks6ZkUzppv7mo+kAXMSrQockQOkIttdzRm1yLxuz1inqRyHFTa71j1yKNzT9I8pnrjc0f2kKZWfaSnAnTQn0k/c5HKVXR9ZmTjvR59N38fG4go2CmKjSN3kRZsGb+x/tKftbUVE0BBSQENMwfKkUJQ5nyVMoib37xd/RX3DRLM0aoVKpuw0zALcWz3ynpd8iP37BppG3BmlkQi2jtvmwjPbBAwel02hP/LRQugLKPyWb6nImLxQ/nAjHHY5pBE6MkVT400MKbfzKoS4iOIQMTH0LTyofl+/mw9iBpXYPX85tl18linMRKYQyd8f7Tgp58Lqe8i++zfNCiPgMmHEriIkUTX/PvvCdL8E3LJkLmoDyfmvC6foem17Tn9QGHCaOBJT6o8lGth++40KZ9mQlg4t2KaZDLrV3axPvxG2baadaNz0gBlD91AZvXSMskKCgGXNCKKrrPpGXxgke/ck/CZNXnhny1jz7lb4RojBFxQembEoOYuMCTJD3jAgenwT7SlQ/T5lGSTSP4t/yis7XccH7LzeQ1+eBeY7S4boOFxPB9gtIMduQbLXznTbnUxiFGBkxMERbvZ8YR4ci+Q7kMyaHJpZYhCUCzKsFyqYmi74gBDD8z557HhM4HjnwN4wveEzfcfm7xgTejtHbedJuZtaDTa6R/vaFvhj3zM70QmABbkMkN5d7QFyvyZapGl/To1z6d0JdwEU16TTsZZeWZNCsRZvLvFoubE1kE5QMBS9hj3v0BkxzqGgysfF6khREaRE00M8xFGdLsMuBwOK9fKN6k1yj6Qm/afU7mTbEPUpQ6uBRAGk7fn04LmjPtJJjBKHUaJfNefD6dJA6eTFFrfHpglqTbtbTAIzhmzczfeVPqcVmvaR5U5+95H5aaTFMkPhNfY6mIpXDeYngT7N2P+UxTBB8/7Oxsa28obNLMhx+8K/F5Fy+c5iLLHMa6+ciZKN6oRzuopQYm6COQyZnzjscR+r2+YCltNNMAt3CUHP5cyIZAdpNMbbByViUyAgzo/yhEftOk3c4HcYf4wAb2J0KZ7DbMNFqwxU2kMNlCMQLmffivgxtiObWlMB5ODlLTAIvPKYhtPFZw5asX3iRzjaYVJg/jOYVwgZLPkQ9upqFEtn707byO/+LrvHX0a+6BBn6+Lzp4rfcZSPCVL348kaOW6Zv6I29WLIS3ZNpLh8BxVUwsR4Lg2RRiYo3cCKcVVvIxnNb7V5/Es0LiTTpNOTeC/pHX401y471Eq2qSOFjO4aweyOeG+YU46PMPSjpTEGo5fbmZKsNqiYPL7I4Glv8SxnMax2ctlQqKtPnlo0ZvOg2rNrDdozoeAPca60F2r3kK1lwAxQ3jJvPv+fl5l2oZOMA187mox80VfI5cFYiCycBK6SC/t8Az+OqXPpEo8tQDmo/pdXvaQCX2gQUyXHw6Wh85Ka1wpSjqg0zeYKhFM/B96jPk7N1GS2NSBmT7wuZwPLQaqqtREg8+CMFJIAQuW6XBJ9weFqxWKw7YN1SKD8n3eP/Ff6vGyo2kho0jZHN5c7MMPpwPcumqRcoU7HAaP/hgZoIhH8iLLeUwKNB8nsFs3KyDcBvXgRt70NS64EFrbzm2WRAftPl80/tbBUXOynjMlpspl/W5T78/EaLgCr6UYkmiq454FEcP7aJRvtZrlddCpZzUQNb0WAZz+aMvFzGloQCYLzDtU/GbIHTWQmsFOw6CU8AShhj0Bsjls0qJ6Bd4fROO0QRd4uv6/YECAvpnasDS0rIKvSa9VnD3PofXbrZamKlZok6AhIvkTTa1c8SAyGV4/r4UGces6hgWy9KUaRHx3Zwsi6J/V6j3AuHNrC8q+GDGgw0H82OP13oXI6AmiSUU3cHASoZuj/h5Ch5d7CEz6x1qsWjAuKWk9iVJYPTu3mC2PC35IfDO8H1hYdHCe2m8h9UNEtTGyXcaTmqbaFWYSdToAp2DyIovv9Fi8AH6gwFazaahJFnDQJke8bo+ifdwo1X3LS3R3fjsg26BQAKDroEJiXzh0CLzyWYSxmMOSezY+eSykDCiRX0Fax6nld9y6Q0FTeC8y6UpFOm0Rb0+mjfEaJqGeT9pEKAVvL2PpgXzRQC5O1ksW8Nev4+CB+1d1hA8/ODHEitvxQbdOcn3dI5Wq6UP5+JxcQwlMrTE7HogLWHk62E/vUbmxHJG0yIzH75WSnMorQ24GMRRBxMzI0y4UNImCjUS3WMoE6oa3pD4KVAQIO9LXhbsqJLigA2jolgu7DfL+7xGvW4luISYdEGaWuQz0no4jeR9q7AgONLhtUw5nJUCn8EJKK/Le83l844qEul6Ucx0y/JUj0AdhCw9O8OjVL4y4tfJR7XSXtaLXR212+vp+lI9F6kH99793mRubg7tdkcPlabvi8bIi3HgTJPyS0aO5hv4veWmKaddzNVYxzOh8ILgE2vjsFho7tMTFocZIUubXSnIJ+SSdppFZxm85bDc1DaLKQ/B7ilc6GkqFt7zPd1OTwHNzMyMQH1dxxWdbYEtDzaNpiuyIMtWKJCpNWTJknRfeKULocXwG6/0yvlHBXqhUT1mZ2cnmukZCcSuD5pSA0Is7bBCufl7Dxh4QZbPdrCe3IyLC7TmjAkGQwSPfOXuxCTaad3QElouvnwWXyQgwSA8zzJQWkBUx6UX9Fm+pkk7z9cSsvMcHl7Ta5aPZKlVSo4dKE5TY4SxSJtJn0BfYeCAmWkvDJ1OV5V93iMFSYGZy/s8xKho0hWPhZg4/DebDjF0uKZ5B/KHFJQjBteCFQw9GcZxgA4rGeMUdnp9bDY62Kh3sbPXRKvfBbPN55w+jOc86TDKmYLez5yU92QRsKVfFGQ+i6+2eAGdQnseQ/a5qwmQ1V4NmJ9fXJi4KUPVQssmfDHj61/+ZOLzH0WzKjtZVCYESP6Si2i8HJpPbgBvloGBoCTV7SxKMzNmGKMiYQVDVnWYSL/XApkvSw8oCMZgc5rlsElek6U549P4CHmqhT5KUeTNao+rnPA6up6LICU0FBSlJxHGCdAfDTEYkvE3RD9K0BlEGIdpXN1rYm8YYbvRxCDJYoQUZmfnUMmFaLRbaLOalC8gmwoxHPTwxBOXsJQe4zd+/Ll6Xp8nWoASy896CNObTwNpjPTFn1n+aJUo/tu/zueSsjYqUxa8gbIypYr+rjL15S/cmRysWmTTVg3nFnpyFj9EVBJXJBYQQF9JuOkAkiPtm9AWXbBDmojjBknrCH0NBxZcOX4RzZWKtu5aRt+cRp80q+LEOBDfhMv8tof85L9d2YjSRLAjIkktAs5t7uNKvYvt7hDdUYT+cIxmt49SuYR0mEI+EyIIs6i3OojTBogXM8Zm6PT6aDTaiFmLdTFApz9EkMRYmZtBLsXy4Qj3f/EreNlzr8etN5zQInPx6XO5GYLyJnwL08Ap9QSi3JRKJSsaOCtv7sqoNN4UMyjjPcvMUqkcOU2fRbNLBMixQgyfjBNdmKgCE+nBgCmBBSs+7DY0wlMeLFywENryNn6Q/dSCE2PBGZTl/cPkbwcuK/dy2ic8UnxVswiWM1pJTjxTS75cnjtFXWjaza8HGMUB7vraRXzykUtojyMsLSzIHOWZMycRmt2BhKdYyCIXptHuG4Hs4vo6arUqitk0Wkw9UhkcXV3FuUsXUS6W9GyDkUF9lUIeWQovEmxvbqK9vYHXvezHlAb6qN3TSBjV+lzVItIpbst4hQVvrb8zNcLKBc4TebIYwCg0Vvmh22FEzg3mWuvn1Ez5DYfG84Lk9zBCEqrvcEWZgUkJxyEOAaPTjBaVacrszOzEpwoyE0Pv20Fpj2jYZnJzzad4xhml3JeqKuWKrqvN4SaGRro2cMEB+NpYXW2iqTuDId7wsS9jvx9LkvuDPiq1qoRy4CovXKj1rR0szc1i3O+iOUqwNDuDVqeN4cgiUfrKdC6LIwvzePzSFeRLJbS6fd1PQYjYWPBnIZ1CpVLCg198CH/8E7fiyOI8AqIyDGTSjMTJwbXareJHuiKBNFZ/NfqIBZR5pod0bSrnuUKFAzXkH10qxI08GPFqBQgacFf5x1flubg0t55WafwaqxfKjDreprfn/qIGPlt5V9priaWkinmRrzeKqUZQgPirY9PxtcZTzUzMr0yHq7bYphuEZmx6q554K8HP5X3sdwZ45QfuR6ZaQyEXStsazRZ6wyFy2Tz6onCyVpvBxSvrmCmX0Gx1MQ4CLM3PYKZSxZW1dTEKIwpOmMZ8pYS52Vl8+RvfxDgxemkhz2cweI1anEoSXL26iVtWivilFzwb/V5b0S6FU8CI4x3T4um5HMTJNeS9+Borg0FlBirYGxzKTaS/9BCl3IjbWB9HaN1NM43DSdvuGWqWVrgKvqocVhe0QrXjuVKbHcxHu28Laj7HKhgGcPuol1rlAeYpXDUNw52NsQpAEEzbHHxN1Zlwbibvg3xZ3iej2lQqg3g8wJsfvIIr7QFm5CqMyNzrD3F5YxuVmRlk0inkHBDQ6w2w32gicDTIYj6H+WoNrU4HO62ekCla/nwmjZlyFReuXsWYwpckyOeyshpz87OosNAwGkgots8/ir/6pRcinfWFcMvHZSYJxijDscqTj2iF9jjgREVtVkLI7iMzXsGFwaNWvLCOAk9CY0DEoElK9tADdwoB8pVxJdf+w13JhSF1uVic8HMMN7UgxZOgLXn3PRvyCi6lmSJGinQdhUSRp8MphRqJqm85ncch+XO+hgGU6nWudqkbn9AzPYifwVo/wRs+9TVhxIdWVxBHrFEC7U4Xjf4Qo3EsCC+JGbil0Ov0MQxYtbAEPBOmUC0Wsbm7g9YwRrlURjoM5Bvru/tYPHQY5554QgKSZd0yiTE/V5MZTqeAze09PPzAQ3jHf/kxpHNWjPagB4VPbRdpK1B4rHlShHbcYg/AywciQLfTNrhTHCcLrAiX+vjDLBVTxhSCz97zPrHz6KcMjWBYbFIlg3mgQcYD79wQaU/KUH5fHVERmlor32Zpii8gKxEOjJ9LtsI0EDJA3PgyJF859oDjClES+Xq+XzRIl8BTan2OK2uRCvHKjz+ExcVVNNrGDCzQX0UxLq9vYWF5GTt7u1iYnbGfx8C3Hn8cZ697Ei5evoRquarNHA/72G/3kcnldf1iMYdsKo1Wu4fa7CwuXLiAQrEkqigXuVIs4OjSvPxuuVrCZ+79Al7/0u9DtZCVj/SCSe2xdMmCQGYMBBaoWbzOQOnLlDvLzfHQoQdvtKGOOOf5Taa4zhI+9MAdiS81WQRlHUoeKAiZebroyf/MXjdltvddbmTRq+WoFAwfWAlQd8AAQ3L+zmO+E21l2uIgQoHsrKw4Tfaht+W2ViP17AVLqyJ8vZHCp89vopDPoDsc4+KFiziysoz1vV2MEWJpYVH4bjweYrZSwn6jjd12D8cOr+LK1XUtarWQw+W1dWRLZRw5tIJHz1/E4sIsmvUmkEqjWqkoeqSw+K9sLoNaMYf5QgGlahGfe+Bh/PrzzuLmU0csonWpmYflCEswK1AuGpH/a5CcLJCDUvl7aj+BfE8CsxzaFa9dbOJxYV6bGy8za1poG2F4q5lJ5Xvkcna6eghGXpQoEqZUkHW5poB5F6gIbHAUCeG8jh7CjyAxi/niZEM8UcxVT6xBydj0MjeO92opkVUsmHr4RRKLIZVgmCrglR96EIuH5tlBJKG4cGlDZnJ7bw8LKwsoZDIC5tc2NrE8O4PzlzdRnqlhplRArpjHzs4uwlQaW40GlpcWMFcp4fLaFjLZtPJPwoFcp8XZOVxaW0OoLq4AxoCNcN3JoyhmsnjwK1/HD14zg397642uQ25sODXrp+qqs3qqcaNoBc0aKaLnOqZDhM698TU9UjdVyzRkjikMQf+N9XXh4TS5pmQxgvs+9b7Et/EZU7ww4eowb6Mj9ugKN4abSimhj/GsPlN15n2xTKyqCNRmtynULO+o1Unm2un4kAUHBhgsx2r7t7cBUvPKpZLgNWN2WgcU/8+Ug+DAG+57HM0khdliCXFCVkCMZqePc+eewNETx1CbrSIgeSydxpWtHfTaXYyzGcyWayhkTIAZbe+3ughzOZRLeVRypHvm8diFi4gccy6IYlRLFWzubiPNnhJe0/WgnDq6ilyYwqUrGyjXL+L/+qkfcHVLZwblPYyLTC3a3d11gmtRuIoLxZJSE+Wm5EOxKE/IznGffGYwiTUcdu7NcHD/vR9UNMsNolobxZ59mBaQeFIR3bGvUfKmbNMth6RZNqCdgO9gsuDeRPi0wTTeeDjOaeo93mf7wqwHMTxDQQ1IB7qo7GGM7v9IK8FHv7GOje0tXHPosCXZwxE29+po93tYWVpGrVy0HDRKsNdqo0XidiqFUjqrtKJUyGEYJ7i4vi1ucDYIUCpa8fr81U3k8tYuQZx1f2cXc4tLkwiS7Iowl8XJI4sopUOsbW3jiQcewJt+/Sdc849lAR6AP1jcNi010pbFRAa4eBcmiibxbw9CqByZSKF8diE2vG8e/uw9tyeiVTiWOTeV5sAHMFxoVg9k3/MFhIS+HH3f+iYst+y0OwLWVe2gTzPWo6SLTUKlYlGO3tM4hXY4NoJn7U0qIGLrkQE4cukJuaE522vxewjdJQpu/vST30CTLQvZInJZpiwRWu029hptLK2uotGo48jKilwEzRZTlFPXnsVes4FcKkSeZg1Ag11ZJHRxk6mVmQzq+3XkZ2awv9+Q0DJN6Xd7KFVraLdayiP7vQEyhRyuObyISjaD/WYTX/zsZ3H7K15sYMfIuEMe/RH7gemc49QS2vS4rOIKh+cpx3StjkR+eF/8TK6hR9mMvmP3LGH73L0f0GYS6poi/aZBMgyumOyxQp+6yE8KUjMaB6kmGW6ma/WWdkUmab4VUJGyq17Q1HjmACNWLowS61zWGnIdnEU/5ptw+VkGV1k7xacutnDPuTXUqmW5ho2rOyiV89jY2sHhw4fkj9bXN7C8vIRoPEKj2UY7SnBsaQE7rTYK6bQKzds7zEFnBfk9sbaGSj6nqLEzHGNxcRFraxvyVc3GPjIUSnZzZXMKqPabLSX9h5dnsVAqIZVL456P34N3/soPWVnLMRJlTRQbWKBjPaCxOuH43Nbid6DFn5guMXKCFy6CVZ7JYoMrWijfcF1n3ODg3nveJ9qIGtlcEOOr/J6/4hF/M1X0i7yBtNh4Qiccf4gsO26i+io9W87xT+kDzGsYDOcrLj7HVeWFyFPecqqUaxGgFZDZcaxxk+gIzSHw6k88jEq1hlwQoNnv4cqVTTC6pHCuriyh1WxhMByp26xWm0Gj00dvPMLR5XmkQnaB9xENIzR6HSzMzePw4gLOXbrMT0ar10euXEEpV8BoYJap0WkjFJCQwvzsLNY3t1T8pplbWZzBTD6LVCaN+z79efzdS251z2EL7pud2Nfi83FRUCZMe99O4TMCo9Co/1IuzjccGV7t6tETZqLU775P356I3iCc1PykbzejeVBV37GwKQls1ElnM9IkI2cZZ9Yzsn01wDe0agMdUWlSKXA0EvNDVtbypTOlLa7xl7/v9yzgGo6YhzGdDBEkKdz+rV2ca/ZRJKthOFDE2eoOwDTpxDVHxYuhWR2Mx9je3UeuUEJX9bCxUgmSwNi5vbPbVAV/eW4WhaxVjLb36tjcbyFfKiAbhAIadnZ2MIysQMznqJbL2NzZFT2zVimz6xfXrMwhFYS4977P450v+35HWeXcgekACwMRLN3jMw/HVmnyQaQxB609cQIUjIzIZiZ1iqyR0c7r+ZwzuP+zH7LURGw0z9IzHHD6ZWiOr4rww2k+va33qQw/3aor0+ER0jzROHxLoEW+AhH0EFNo0My6J23Y6yIWHjWEwfBYPujl9hB///kn9PtKqYR6s4nLVzYEtS0tLqBUyqFaLqmqwMBma3sffZqqbA7ztYpKXkRvcvkSHjl/AfPVCor5LIrsscllsd3sKFBSkZ1sCiToE15j9xiHS6QN5OCt0eKUSBYPElx7bFk+/d57P4e/fclz5JPZQk/3ZQtu9MhJXKGAx1KWXn9gRXYBI8bSU+whX016i60yr8Mo3gjhrp3D85O/8PmPaDMnvBQPYLNXRH0TBpT7CzH1oHkw6THUSMk8AWPX3xhhWtdkAEAfw7sxMNkEw7TSTEA72gUAACAASURBVCi/PLuAhWr6UsJefNl45ArgDkToRRH+7rOPI86VQLYBAyxq3i61L5/HsaNHcOnyJVx78oSChXq7i6vrW5hdWrCUih1m6RD1dlsBVGswwiw1MJNGnpR/ggLdIQYxKyJp5NNptLsdLCwuYWt7RwJN1Gev2UKxVFLuTJdRKOZxYnlG/N7P3vs5vOYnb0Y1n8PYbb6UwTkasR4c8TuOjcWRiN1gHFyXnBuCNJlhYOtG1+ezD8s2fAtIguCeu9+b+EBGC+t65qeNKyyu+tbtaZu73xAuEIMZ9VlQEsltdRVw3z5gJsR4pboRB/mZtE7rkso1M1lJr8cgPX1fZgkJPnO5hXvPbeDQoSUl9c1WB02mG80GbnnqzYoG165exfzcrIKbK5vb0qaVlSU0Wh1UKyUxBNa2dpEv5tWcS/tAE0vh2dprYn5hXmADNSKfzmCv08JcbRb79X3DQJHCSHXfMnqdruDGYimH5bkq+t0uHv3yQ3jDz9yKuVJJSb9aCEaszxqgbsUK6yILUlaYp5DwuQkVivRNRN4PpEhM2bh2W1tbLkrmdBPXdOvSmeCzn3m/gHamER77NBTI2FPsKmavvtcsZ5GdH+Um2bAEBU1i2RlpiwIgaNAFPhY+m0bz4STRzqmLu+MCK0Z8zCt9G6Evp/E1a+0h/uKOL+LM6dPo9nvY2Klje3tXlfobnnRWheIoIAV0gLW1daysLGNjdw9HVi3X3K63RK/sDfpododYmK2ikM1hfWcHM4Uimj0OjEgwO1PFbqPB0EsL3We0DTb2cgNGCo6CMC2EiZvJ6JvmeXG2imjYx6NfuBd/87IXCHhguwa1TQQ4VROYrpDJzpRlhGptVv6wXq9Lb0uVyoG805IKKhbLd8ak8DOIpuN9KMBMH4NP3/1ebSZRfPJmKSHGGnBNPa7Pwie9PkDiJvo6qEo6rh9EJtIRjdSO5/sMXeIrIODAVCzPSHAWSAQsaidrnXL4hl5gMErw2k98BZXFZYHcm3tt7DcaIGWSwnP9tacRR+wgS6tFcH1jW9FVpVbG0lwNGQ5H6pFIPMZOsymcNZtikTmnrmwyCgg0sJ2uUMipI6w3GGLfsQDoLmiOuQE7jbbuLZ8vGPtBPShpBNEYhw8t4Wt3vR+vf9kPKSrmevi+HAU3qtumJ3VaBkBqOBK31nJ4tWtQi7mOftKZawk04N6SNQMaLPgU++9f7nqXek1YMffFaV/T9LbZ55v82zPoPEvO56bSXFcZF3dIVESbJkJHbjmWm8XDsWsqyPrBSNbhJe2VYzEw3vsEsgM+dK6BvWGCvXrdFn6/KcYa0w/SPAie5ws5PccwirG+uS1WwXVnz6BSNE0nXW2z3kan30O1VFBBOecmZa3v1jGO6FKYGhH6y6Ld66Pe6U4qNTHfNzMjrabUk5HhqyG8ddY9a5USzt39Abz1N39KPSA+E/DBZOw6zZRqcayM4oMQo7GlHlZASAkLtgjDas3MDjzrkCQ01lIVx8jysV9mhOBepiYORVB06Ro5+b0nEk2BA4PtrAXAODrSrDH7EwcyJWqR921yjjXAmxVrbTCUCWWLva+IaCQK647yq6HBVMJeE4zVuRzg0+s9XNzYR75YxjcevwCkstjZ38P+/j6uv/46tMiYazSxtDiHVJjG1k4d+/UdnD1zHcbxGJV8Fvl8FjvtPjo98pwiVKrWmlDNZbDfH2BrZ09QHs0p+Tpk7JGFx2iTr2MBnJ8xv7SEnb06MmxnKOQwHljqRu0oMscFsPfle/Cml79wCoC7gM8HjbweKSlcs53dHRw+dBj9KMLszAxYMKdGZnMFWTCVGxlAOr9JK1IolieNUMrbfTT7+fs+mHDTGLQQgaedE7HW5X4WyZLawLCds3emA5PoCyhNI8dtNVDYSMDe59HMaICT62Dm9XJZMr2tomJMd4uWFRFzdh+5u2Zo8MFvbaMVZzFTLeHKzr7w0831bWGti4tLKFeKQp8uX17DyWuOioC2tr6Jm248qy6Mxy9dxKGlJX3Gld06jh45iq5gMdJIIyRRgq16A4tLi2IuFDnCLAyxvrON1dUjuHJ1Q89CtIiAAzVza2tH6cjA0SUpeDSzuXSAeNAHLn8Nv/p91wkoUFuko6cKnHGMDaZR0+cHkpAkcetYV04pzhBthHsdUhJaXqtSnbHCvhtkxZcowORmeqfK4KXgZud5DisX2XNaadt9sktw3fdBaPKWy4O0Bb75yPFpfeRLTFKkZjdLyPNtFblmyXAnWE/2QoL9OI2/+eTXcObMNVL/9mCMC2s7aDSb2N7aVqR66swZ1Bt1fbZY7oO+zM1crYYjK4syp2s7e+h3RyrLZbMh5ufnFKQ1Gg0RkpscJDEeY2l+Dt1ORwy8equLXsTrzCgwYZ5crlawU7d5QJ1mA8VyGf0R6Y4M8kYqPJQKGew/8TiOl/v4zR+42dI6B7LX9/cFDZqrYTea665WFYhLQkWIrbQm5Md4PvSJ/cEQ1UoVnS7pIUbm5jPIDWkWxRDLy8tQNOvNpbTDtY77iogH3Pk3/aWn/RkYb+aT9Hivzco93YQval9Jc4TMHlsngHFhzF+yD8RQJAYvUZBGd5Tgnsd28OCFqzh24hrUW8YtGiXAxtauhGF3y9KNa665ZjKyhvjl5sYGKuUybrzhLIa9njivO60Oup0+gnQGc3M18V0JxBMpYqkslc8jl8tgtloRQEAt3GowhyTx2nVuj0bYbrSRzReFk5LM1ev2MYwhLhBhwTSDrXIWV770OTznycfx87ee0Wv5jKxyEA4slctuNh5RIJv3MDM3LwBj0B+5EXRUGE4mSyuNIWZbrpAFkUGsxienke5vxiZMjWRqP37nO6WZqjOyVukwWgMEOGNupNTEEJspuODJukr4CQyQj+or5Z7aIZTIsExKGE2ubaqVhAhU25i1NOrjBF+4Usd9X30cZ649i86QvY1D7DW7uHDhojaWKUi33USj1UI2lcXM3CxKlbIbkDjA5vombrj+LJaXZtBodNDu9rC2saPXcVHoElT0HvRRKFcQiSYyQj6dlclKRmMsLC1hr9VQAMT+TGoF06xdfmYmK/SlVqxgr9lWGY4pw3Dcx2y1jN7+LgYXHsYzbroe/+Gm1ckMBJlWQ8XNPB6Y59frjZArFdWJpiBHLR8W8VNT2Z6QCjOa8Ml4gKaYxQjlrW5oZECMikpC0EDDIdyHcK6AmUlDbHwHtYXXvpV8OkJFqD2FQB1aRg+xTTO0gteZSLgzxQLp4wSNYYKL+0N87vwatvc7OHHqpJLsYZTg6996HE++8Uace/xx1VmZVnAs2/raOk6cvEZQ3aXzF3Dy7BlJ+O7uNm556tPQbjUxWyui3x/i4uU1jKIAC8uLaDaaWhj6Q3aczczPg7K3t7Nrsxjor3NZHDpyxEwYn4fROAnYuSx2m22ZFsYXtXJVcB/LhgJUUkApF2L3G1/EmUPzWJ4r4/+45ZhbQ2PnMcXwLsoLPe+buEmpVlXFhEwIQoYMEkVxccOYyUBQ4Ji1EiOtmno+w5TydVoY0Tfv/sT/sjzToTRpsd4MCPBBi889Lfix0SV8DzfYd0Lz5xowMRnpMmUMeIYAzUSzn+CRzQbu/foFXG32MVsr46Yn34jeaIj17X1s79aVbuw2mjh85Aj67bY+a3d3R34lky+gNjOjNGjj6lUsLy3Lr83MVrG8siTfyXti7fGJS1d0j9VSUcyI/WZduGq33UNWuWSMIaG7bs8i8WoZ3d4Is7NV7Nfb6I0GmJ+dwczSivLZdpfz8dKI2J09sPUhZsxKzWjrEpL9NTztlpuRG7fxwutWDI50gy74Gs/Wk1b5Dm8OZ5LAZ1CbqU2GOAeBNQZRown9Wc+MpTOexSiMXLMWHCn9rjvfmVinsw1bopk18MCPIfX4qQ1+8jwWT4zmwnk2uSd/eQzSg/PNKMD9F/dx/yPn0RgkmKnVsHpoRdTEQ4eWsdtsYm+/hW6vK8Rkf3MbxdlZm3unslsE9okSfz1x6rTRUmiKWN5qtSSt15w8rojVF7q52fvtFoa9PpbnZ9UyEI2H6LdbKJeKjtvUwkK5gqViGoj6WKYGkzqSyeDKfguPXtnFoVNn0eoPEAUJGs2uFny/3VNEThfEzUz16tj91pfw3O9+NgrJGNlgiBfdePwAGsY6rxvq4eg1xIWtLS/kODQpiE0Ns6ZbRuKamcT/EXLU3B8378HNqbVaJufvmosMPvGxf9SIUm9CmXRbsOOGALuUwYME/udSc/7O5Tga0uD4OSPXMbablHDHw49ju9lFtlzD4tISOr0u9psdwU8bG5s4cuQIrm5sSGqJf4zZkdXtYJTJqa+SsV4wHODK+lWE2SJqszOGSbIBdzDE2uUrihIXF+elwa1OU+ae6NPe5hbaOztIohHyqQjPu+Usbj4yh3I+jflSHsVyCUE8Qj7rmYbT2X2Ufs4+2GoN8Y3NNj722Db2esDx4ydxZXt3knKE/SZ2v/ll3PLMp2KuUkAw7iKXGuKFN550NJq+UVIdOY3fW6Jv2GxIgL9AZMmK0SPXKslJmRpkJSvoOLPslSHbIwxFjGN50Mhgbj7QXXf8Q+L9oar4zuSaGXVjvA6kEhbdmlpnWJpxZpdSyvCZEewwDnD7N3ew2egjW+Jk6QzW9/awvbmrmT/MnhjOl6ozGPR6AqcNhUph68oaFo8fQ6PBCn5OkWNjewvZSk3oDstdbA5mxLyxtoalxSWlGZUqGYMZNPdZY0yQyWex9fg5lKM+fvlFz8N3Pf1JKGbVPwim4jF7PFiVGA3ceBvF8jbn3bVYiMCmSSQ51Xs/88QePvBYD8ZyChD029g+9zU865lPRbFUQDLoIA1SWIDvPb4gBWEdVhxftRQYYY5oF82qrItr+eD+MqckX5eBHz/TdRtPgAubPz/tLLAhU0bTZBwgOI8SIMCAUdaBeQBGtDJmtuA1aqwLbmyzra6n6SFia4cYjBN8YmOEtb0Bzl+8iHyxhGbbBjkQfmPUy5IYA5LVo0fRaTUn6FEyGIFLSfYA+x7VgRaGohXSvPL7zbV1oTes1IyiCMsrK4pC63t7YrDbNWJkx3387PfehBd8xw0qzbHBNlaFnvNuCaiz49hmAHW7hrWGadskPiujVj6jEC9QSylwGey0x3j9g7vY29xGajzA0295Cu0Juu0G0nGEfCbCYi7A866/xvk2izp5LSqCH01OReG6sTA+IngxJo6bRTqX0XTNdCavoIfRldoTGeQ44l2vO1COb/P0p6NhBbQzbDf/prYtN6aT7XyWOvAhZF4dScsIuX7ENOE52nT70I9dGeKf77oP+UoVG+ubKJTL6pCygYjWP0FflyvklSBTQ6hJNK3tdheLRw4rR6R5bTXa2N/axaEzp1WxYEjfbXeMQUAGfDaPaqWIcr6IXZlTSztm4j5e/cv/BkuzHCnjTWeAXrejvDAVOLPk/LH1TlrHNglWisY1u8ANQxwxV+wqLXisncFf3fFVPPmG0zh2aAXt/S2M+j0k8QjBeIRaIcCRWh7POHHIaDhJpGf2AabYBZo2ZpOsGdwME7oYFihymrbFqg/IEWJRggElAqVFaQ13tsoONZzvZxTsp6sFd3z47QLaDeS2hhbfa+KnGvv0gukHN0JsPkd9kHGKE9nwRj/Gf/2ne7GySDb4BU3rKFeromgwZ1P373CIer2D1ROHMezbsPhRv4v6zh5yM7Mo5Gx+LP/sbW6gPUxw4swpm8VOs9TriS03TGJUa1V1VQfJCMGgqzTkRLqF//aSH3Wzcy140mwCTUIhQO64NcxLYnJsmYS7Obg6QcJmrXuQX2kAc77xEJ/biPHWex7FkdUl3PSU67G/cQlJt4GMgocxUvFAbQknagVcvzKvaxB3JiatYE7z5k2QJtUk1yTV7Y+wsLCgjnYWyMlG9J1hsWbU8ogQg/esW9CYGr6XRSQxggZealQcFsPapitSlQ9yczTCpdeb8GvtHBTTWtrv/SSPl7/h/VhZXcEoCRSgsNWc+SG5uGTIMSjJFSvI1UpIB6GIye36vgCBbHUGJRK6KK3EW8+dQ2XlMBZXl2XeeU/1rW2L+JBgaXlJDPZer4Vofwc3r1TwOy/9McR05a5AzmCDn8vN3NvdNvagnCJ313pecnlrxGEbnRXOrdrD/1gjzxBf62fxDw81sHPhcXzPD78A3f0dxM0dZKM+406kkjFyaVZbAtxyZAUnl2a0mZ0OSWWc30M2gmUJPkXh35msTaoejKxRSd3e4gllJFjiJ8tPAo1222YiuJN4VF1RekIeUGQ+U2i+M6MM6fmcuYxNc/Y8HV9Y9rir7/VQCqNWtZTyxpf/zUdxw41PxtY+Gds5tTaQGKVCda+HRruL1cOH0Wm3NPqFi7t96QJmjxzDoMPBDjmEQYKrjz2GleuepIXlRlfKJfT266pkzC4sIHYz2+PBAO2tK3jSQhp/9J//g9UKD/CVNEWM4MeIfSbcyLEAdoEkjkNDYhT9kw9UrBQ0pWmMwwxe+aUhNi5cRHtnC9/9g89Hf38bQb+JYNBBPpUgmx4jHRi8d8uRORyb42am0B/YEGEKFeMF/s2R5+Q2sYTG2my90cBwYG3tBO8prKHzmcsrqzKv3FjWPEmFIWnMz42Q2XZ8LIEGxuM0Mq3Sg/EYxTzDZTvgxQhYzNMYGpvT5Rclz7dhUzsb3RF+5R1349DqYXQGhn3yWvSlnEPXaTYR5EqYq5YV4DB/Gjq+6OzSEqL+EM1WUxSOyxcv49qbb9b9kBlXKuawu72L6syczPag3bVgorWNamqEN/32S4T6qJXO1S7ldMjSI8Afk8NKLDFCdtwSmJ8JSfBmbm2+UX+7Eag2/TIlYXzX+QRfuNrA4PIVlFZXcGh1AbloAHSbSI3bKGVTSIeslkIco++74RqU1bLD4VE9pRNEiSiUvouaVk0mngM+VOu1uEOVEo2J4fccB0sucV7+m3VMC9QoeEbmYvzA9IaBWvDB29886ZzWpoppQF4KAXPepG+QtSiPFH9WGdj/oaBHQILBXilEeM0nH8MXvvEEyvNz2NraFUQmRhslP4EoGWS78UHIDm+3W6gtLIGIpIjK9To6zTYKMzOoVMqKQhNSNdi8ky8i7c76oL9jG8HSbAnfceO1WJyZxdVmA9WZBeQ17tTY9PuNOmZrMxq0a3PXjRFI87nZaIqcRd+t6BwR0sOOhlsVghFWSkI98dqv9lHf38H5Bx/Cd/7A96PTqqMUdxGOegjjnoSPTBsKA0lhP3rzGRQyNq89cicS+UDIt/l5nxmm7IwVDshQwKlJYVnuolgTvM+s6+thaqKDguhDWSUa+gnb1kIffPxj/2glMDeMiJspAMGB4Yr+DpzlYXnN2LHITIupueoYSyW4sDPAb//dh3HtTTfh6vqmURqzFokRwsqFrqNrPEar1QSyRdUGg2SsUlNjcxODMVBZYACRQpgk6O7tYJikcPjEURw7sqromMjP0UOrKBdY6TD/xla+kjtSKRuSomit+Ht7DQVoZOAxH2uSJiKcOY3ecIzlmao18UQJ4lSEZr0llkGWfj4CHt5uYtjYx/bGNk6ePoHUsId0v4kM/WU8QLHAyDSSe+BmPu/UiqozGtXmxusoOm+33RQS62mli2L6RW09duKUoW4KLEOk2JikwwYSaS/XsdXpmgbCymCpwAjhfiLJJACiBIgm4toSyI2hCTVfadxOaqYVT/1ESuv7sNk3dNpEKlJ42d9+DCfOnMXFq+uTScaDcYxypYQwiGVWRr0u9vbrKM8t6IAy8nHiQQ8bFy6gtnJUgRPpIBkJzxC3PPuZImWR30rtbHd6uqe5ckkIjuW6Mc5fvqKokP0iLADI5FIwkwTt3gCLtZK+Zw5NNvqj55/A3OwcarUKwJlAmk6WE4BNljyFKFOdxcXHHkNnGKNSLqAwaiEctBFGA6STsZqMIgxRYA6dCvGip50x2IGpVI+Nv0BPM2XZkOWDKjes2eegTP/CnCZLKQALLO+Xn8znRGDTNM5MFvlCUVWgbCY/gQx5KEJw50dvU0sfN1HTMNwIbuWCPNtKxGPbTBaT1eXFIe9yyvw+pYjWuLRE8yO8+6F1fP6RS+ix4kAuTbeNuflFzZHjTIEgirC9voHS7JyA7yHLPEiwf+USkkweK0ePYGlhDqdOn0SxmFdl/8jhZczxfA83XKQ7HuPylXUcP3IIIZNu5x81rInzcti7qNQgAsP+i1evYrvVxeljR5BOrKDLiSGE0vbIxMvmUM4V1ALf6ds5JBSycqmC5ePH8PCXHkJ9AJSyAQrDPYTjPsFhZANOJskhDsbyl6k4wr9/9k02fZJMwV5XG9hxBQNuLD9bcUmxqEiX7RM0qYVCCaEbVsEZDRkGgyzwMxKv7yvf5F7QvIrwhlA4OjeW+ad8php2XJOtgAPHHKfxIowlkzThsUwrLH6urCcD+cagr2718Yd//2GsnjmDQW8EkqKJp7LFXDSTZkM9j0z6Meii12qab+538bRbn4MnXXcKhXxagsUGoksb26hWy6gQ//XHLaWAZrsnNl2RqYWbBc/7J3UykyuqjLS33xByxXYCjvgk2+6mM9fIEvC+yVTf2NlGd5RCj8k7cVDXds8N6TabuOUZz8AnPvkpDMIilqpZBK0NhExrRkPk0oxgMwjSJIGnkIki/PDN16vYTkvBtncPyAgFcnRTbqisoa8qsruGayAEilqaVZ8Mgye+hopGQbWMya7pp5FRncXO+9hH3pEIDBB1w+a9MWlW6uF8qbH0/KcaUsT5cBz+ZFQSBkJG8OI1+lGIn/uLf8Lx665HvdXTnDrVMIl7xjG2r1yWec0GCY4dXsTJE8dxaHkJfW52No8CzWZgKQ+plt3+EFEYYpYDI4RtWPWg2WyjMxphYa4mfytCNQcgDga4slNHPwpwfG5WRWSNHB30sdNoYGlxHiWW7zJpXNnYxjAK5M9khXicFflBvFoKYh+cPH0SH7z9w5g5fgLlZIi4vSUTS2plIWMzGcJ0oqArH8R40bOfoXZ7G13qJ0a7IfvW46FcXVmCqyXT76tznfEFZysxT9eQY6ukkEIi0F0Yr3GO6FNJm+F7mccHH3n/WzWjfXpCrU3DsgYebpI5aN/0Q4kwTJBY4pQ+yYWctHWHKbzhrq/hW+sNZGuzAseptamoj72rVwQcnzx5DV7wfc9FqZhRGwBjTLHh4gDlfEaBhDBNmOM/d+kKrj95EhCTz7invL+9DnPQiiJvBlTs9CKYzxk/6WIV5RyxYOgz2PqXT4W4srODbLmM7Z0ddLs2XobBSj4MUCgV0GI1QnNuhyDf7tobzuLdb38Xjj35KShwE/t1hKM+UglNNYdMMXm3sejzhQx+6BlPE+DPtaJ5pYJMD6C1w+n8YUCe8KXp6BpgzAI1/TmzBOc33YxfpiQat6qZhgnqjeZkr+TyPvDeN2ncmp22ZxNGLEMyDdCgJXcEk2ez+yledtaVG4Srg07txDimLo9t9/H777gTNz79GTh/4bLMdTkd4TnPfqomeRH5KPBUIR1CYNO1yBQnqMCuqlRkB7uYhQ9wfm0Dh1dWUaL5JZFY7XAJLm3uok64LM3INyWgWg9ab2B7dw/pShVH52cw7PPUwDwGvT7Wt7dRJA2D7Xqc6twfGOTGYVHxSMMQU5kcKs58Hz60jNve+o848/SnIzPoIunXkUv6yCJCPstYggvGMRgBjs3P4TtOHbNTGnRU8hANNva6Q9+I1nDhGVVz/by55TPR0rFdgZUU5ujEZ2k96A+p0DNzcwaJBilsbW6JRrLASZcxJ1s3/WZa5GVjSd2AisnYl2kkS2206rklr7lcwZVr0kI2otj4QmoFHMX4lTffjZXjJ5HOBbj5yU/G8lxRvooOP5MtyH/QHNFscN4OJ3pwpIuaeEIb2ivAO47dUKYaSlmjnDBA4dwCMtZaI+sZzXJAqJu3w2iXk6ORr2C+RjCe9H5GwW0MugOMhl3EubKxyNUkxD4XVoXos0IUS2V1U7Mb+/DCAt765ttww63PRapTRzBuAr0magXGGrws1SqSSb5+9RCefHxV5TxqZL2+Z01WBCU4FWRg5GVuKIVVwAtHdnd5HhknkqVV82U3HBuTaGoJhghy5bEegwGabeMzLa2s6v0s6Av0+diH3+EGIVqjQJ+QmvidFjmxZETtIwnYjt+1AX3CMh2MxA9SusLjlSIoQmU09tmtGA2wTc1wVeo7R1GPhgPkKmWoDhNzzDZl2uiSaxtbmF9aQNmV1zR+TcdWjdHsDzXAgVzWUWImHsMh1teuora6ogkhTNKpsaT9j3luyHiMbhKCeSf7OI1pHyj/a/OoxUIFRxc5jYRz3rvuzEzirFk8fuECDh85imuOHsJb3vR2nL7lFuQGbaRGHYQjcmwJe3qELBHwcevpYzg8N28gioB14xFzfSxC5nnZNLW9yZQtz4RUgMShkUNrpmVUTp4u806W/Bh68jV+0gkLADak0tYo+ND7GM3aOBYd8eQaZz1Bl0MZfLuAzayzRhZNcXbf+0Yj6lKf1flgBhf7KWSCGJ0oJfCcksMgRNKXABeuruPY4UPaTEoeLTynTxPWypZyyLgRb5q8MR6j0e3hrs88gCMnT2pciwSPZ1YSlRpHOHRoFetbuwZ7aU6fkbr7zTqG6RyqczOoim0YYTAeqC2BjUbNLseS5mWmeb9KylMWxZOLxCbe53zHLXjz37wN1z3rmQg7DST9JtLjLgrczLSzKnRViPHca0/gGIf960QDtg/YSUQeMiURjYX5VtvquHRL1Err4bRTHVjWotvT2Bg3GpYRK7m7ml3rOshIxbSTjKxEps3kRXOk+amH0HBKXtxHtf6YBp9v2t+WpPN1VKvxYIxGYQFf3o2pmsgGsRakQ4XViGVSIOgLRqBbC8Oi6Pyc4xMSydDotgCXr6whV6mhWspbt5S4PB0M+yP1Yy6tHlLIXm/uuyG91mOToQAAIABJREFUFnFur11FML+ImWJBM/TEZSrkBSjkeD+FKrb3G+jz+ENlbNZFTdRmtz8UN7VGkpdGgltXG6/B2uPS/Dxuu+2f8Izv+W6E3TrCfgvBqK1Bi5kUC/dWveCsn2cenkXWsp7J8EPNt3cFb/puOyXetXQQGi2XUS5XLd1wvGIJv4YoEkTIYnd3D9l8TiU/wqIUDvaNWnCVFvARfPj2t6g9oejQCSb2NtvAaCOeK2v+0gB3fwK7BT+UzBQeSx/CY7sDJBoEkqCYDpEnuEx/xmnOuZzY5py3c/6xR1GozeMEE/iAeLA1EFlOGwqWIzmZAUynS2SKJnOAnc0tVOYXRWgOYwLPxDKBuD8CohFqC4sKatgZzZYJHRsVjTQutNHuIShXUSaOqlTLfCVZ8CJt5wqYrVUxHvB8LTuBiALIfpZrz5zGW95yG45edxaz6Rhhr4l0zNMLQgdP2vWITb/wqU+S37W2xb6CQWHajsrJKJlBz2Bo49X45Rn9GkXHdKdQsNSF7kw8Wlong/rEjOjZYW5MYwjmjIYRypUygjs++DZtJhfU+0BuoBVpzfx6ygOBb2sfcOdOKhhK8Hh2FQ9eaWg+Oaclc9MXq0VEpH6kChogoUlaqqJE4uJcXNtAdXYO5RBCYeiTGWkSYiNSs9YaIiCE5XJTsdN0Wm6M3PwSijr8LBDYwQXrtzto7e0hv3pY5o5IzJQ9ESHNgCkIMVupaJCEigmu6jCORxp90xgHKOVLKMl8UkuAx89dxPc85+l44xvfimufdgtyURelqIdU1EM2lQjcEAacIlCf4AdvOCUs2tI5junuTDqiTRmm53lpzg9dgSavKJLSerOnRJ0DOvyV8xzY/lDS/bCeyaYmXrsf2Rxb1o3JwA/u/NDbtZluPp8LeqxfxM9FpwAZMG2ggL4jKJwKsV1axt3n62j1SDtMieZPTinNTy2fx0Z3gJT6P0eIR9bmvVAtostpD2FG5phWeDCOZAY3VLwu28LSQpDk5M7K1PyuUQ+52XnN3+EYFpo20Qwp4d0eYob3DPM1yozReSAzS4SIJfpRSDyzb5O1JqciGbzHoRTDJMTyvE3u6rS7OPfYRaVTH/3AB3H0hqcgF/VQGLWBURflQhqZkO2KgiuwWCng+Tec/rYZd72++UNbMvPzPp3jv7n2xuOxiFcsf3+iLoNClhAFKNA5pKxtImXxCjdTA4YdRyt4922vTUR2dsfR6zgMN6LUIlp3AjnhPjuKYDLxgqHyY7lrcN+5TWlWZzCQ8261Ozh5eAmrtSI2Gm2102XTbJNnYJHIp9A8cy5szWG8e/U2Rgp6LJBIirOC/8hsENuBkTRTgPEY+WIFkZL8xLXe2+Ap+ji+p7a8IkCf+LKnoHDBWTxmHtsPs5gv8gT19CQlEP0iCLDf4PyCBWkbc88LTzyB77r1Gfjo7e/D6tkbkRv3kIo70k7644ACpYN0A3znmeNYrVjBXSRyB/4T5aGF4SYa8uPPYDnY7mGkcZLeRH52Z5/RtLKVgga51bQTlTjtxTR8Ot1LJbDb/+mNmpLkD1sRdcRFX8pt3NARSr5KYa5dnZvKDemu3oQHzl3GY/s9NJQrRSjzNKB0oGAE2YwOxabU5cn3zKawVGLJKMQjW02B3oSpbGAwMOYpRq0mxgU2+bB670jYGtrLxNymlhRr85gp5hQ9a4IY74e57qCDOMyhx0ZaDgqWQPIR7XiqbJRgdxSjxgGIjpHoz+wkhMh+y6tbe5iZq2HY5fy9c3jRjzwfH/inf8bMydOoBGPEgybKcR/FvPgpuvZsLsStx1cwjmxgRTZbmAw4FqLmmou9dnpLR0GlAvkRBBoK7IrScnE6q4z5KQmeaeXxPedv6fKsBJmS+Q3e9bY/T8jR4Q3xA8YDknZTk7MwlQP5kw1cFGsNnkzUgXpmBo3SUeSKJXzl0ha22x0MekPEqQD5HCc0ZtHsUqLI9+E88yyKmQS1UglP7DSUU/WFq7IHMlShN+53MCpUUG92UEzzlII5tYcrwut3FWDkSlW0OsR9+whda72ETzSRMQaZHPJMP5jyZBjCc65AREhGYEU3JrCdiHRNqgaH7jMqtVYIC7zylSIeuf9LeOkvvBgf/efbUT1+GoWohaDfQik08rQ4Q6kYzzoyi5WZinJoCn6oxiMm9EYbMboHuTzWsk6fKAqOG9tNq+Db9wxxY55qgROBEGkeAz/ORBK1x47NsrlB7qzsOz/wlkTEWhi2SNuvHNP7Sfp2d+qeHRnFi9h5J9TmYZLF354bYblaxlK1gLnFefT7I2w327i8tYswW8D6Lsd/hho4WM0XEaditJttzbzjx9lZKoFaEWje5ktp5KrzMnnLs2UUwpRON9AYbxEqEmQKRY3eZjTMGqJACc1DCJFKIqRzRQELaWoO2wXHnEtn7yWJrN7uI18pYUwcNhVrM1UtSQVoNJq4sraJ+eUFfPPBh/GSn/+PuPeuT6By6AjC/h6CYRfl9Bh5+o0gwKFaAS+4/rAB9TwOy+gAzs9ZtDqFSP1hOabB/Dzr3XGUUHWP0xwaKMINZU2Tm6sGXfpKHj6gmGbadSDY88Pv+WvNzqM54034yJUmx4ZQeKKzoQ+e/a7FJ0kLKbzlMccxTWeEIFUKGRw9vIqV+Vm9p+k2t6GJkozSWImDyj3Npm2QMek5VSOLudkZzQa4vLmLUjZEhcVfnQFNrUyDhSIm/ft9S2vSKZtNQHNFMzUcdZHhSUFxiHEyFriuh9XicHDVWAD4/NwitpoNpFmHpS/mIEXWHltd0WF4v+1eF6leA3OVMspLh5B095AZd1DOErcmcyKF7z0zj2qa2jgdmGzHx9gXr+mZ5/7fDHjswDrmnDaDViUz9mGqVY/jSdMikVPLbdq1+VpRMCksrhtdGDCDwPe/+7U2otR13Poh+Qw2zCwYYOxLYD68ptlkzwtGY/zD9pwNaiASUchjd68BG4lLAlgGy+Uyjp84ovk7LLTuk6XX7Kn0tL7XkJTRBLOhh6D0Xr2J5dkq6p2B6pX5jPl0a9JNBMKz7pMu1KRtDHao3b7hN0lGyLAdLsO+yo6gQU4bUcM9WQcaIzfAqD/W4TNMYzRJWXMDYgxGfb2u0+qw4Ilo7wIqCwuoHj6FoL+viLac5aSuFIa7e3jxrSdE86ArMLKbGwbsGA06AYKnLrjNsC32g4SNu2sbTnNqfCoNEhYVx47UEoFrctqEEb8mh80xaCS78rY3/oGRoF2OIzOuQRVm03X6gcs3qf6eeik154cFAT6PY/jGlW0VT9XS505dJDubqQiJW0xyWbXnAPnDC1WcPnFMdp+MMw5I6o/GuLpLVIcIDFRNqfeHKLkpYcT/SWVhpKiRLewBSaWx0e7IzLI1gLtF3i83jtrLCJb0T7mMeIRiPi86CNMQNumwBqsWAM7fYY/HaIh2q62Oaz4fZyfke5uoZBJ0+hGKR08hF/WRizqoELcfj3D73/09/ux3f06z3/1se5vk6doG3KJ7Nt0Eh3VHavWHlgEouBTGPTXLLHUxl9D5nlorDgHhJtroGaFOkwktNLPvfo0b6+3MgaMbMkUwtH96xpbZaZosIwmz9MPzQDYwjy9sB3iCgwEFR1lXFVngjL7YWsCjeKlxG5vbaoOTVCUBBt02jh86jGtPnxAmyiCgN0ywu7eH3U5/OsItHqJWrqi2KbgxHaBWKOBqvSerUiqY32TQw2uwmsEN51le7DqjdpNtwPtmPycXjmkCUZdjR49i1BvogBpyWjksmPTO7vZlnF4syrdxgFRh5RqUsjGK4x5quQAP3H0PHv3KV/Gbv/jj+K5n3az7Jx7MaxODVSSqQRI8M8w4P0Yqnx7eRhqqby9QK19q2tSszbVQSGZa40o1A8iOxuAH6VmJ39Jy3X7bn7mWPotmdXSv+5JfdFVVYxtMTzI3k2BdSTTD38xdi8e36uiNh7i63TQ+kYjjgXU+sQdURQ52UwcKQhiVjeKxonsdBDoa6vSe68+cwKpOpg3QoA9kDbA/wtZeXQdFy8fQp4jSnFJ+u8TR3VwYBVWsjNh0MA6+ILzAcliKI9JIW3THboxGLD2RkW5DkOv7DcSZEI3dOrr1bRwqDDFXKcrkrW/uo5UUcGi5hmpqgMHeJj7yzv8lk/jsp12HP/itn5uMG7cI0gBaTVUB0GxwNoPvOLfZPra5brKLmw/kqZRcvZgmRRNZeFKFrbUCIWmnNTlZ2mVBanDHe/5Kmsnyj3ibOmQ0P2GGHzxkhq/zBGhr9zMBsdMSsthIz+HyII/Pf/OKIRuUFgZX7mhGP7CyUiiq2sGb8Qd8KqR3kk22AXPPve1NLFTKOH7kKCqzZZW2xolxZTr9vnpZWH3fbdQNUiMTT/PfA1TZSUbfyMGBIcN5I1xpBhYDN7XB8dC2looELAw3+l1c+OajGGys4ezpJY0yzbE6lErh8tUdbLTGuO7MUczGHXzgrW9V7sdFYP31LX/+m4r0xYd1BwOYMFtK5U9w943Cvp3dayphO8F33DjtoZ9CYt8b19eoPZq354IfbaY/puuO97w2saKokSzVsqfJk1MIT4rtbso6o3gxM7+W/DrzS2lKBfj67hifvdDS0AlBau64KEqUehRzNrSiRAKyY9KxLMT9YH8L+zuvbGyJDsKbZkrC6FxzetKh2uPnZqroDvq6tgYvCngfimHHC63vbJlPV///WOaK6QfHi9M7kW7JA9roJ3vNDi5dvID23h5mczEWqgWU8hnkWKwO7fztb17YxCCVwXWHZ/EDp0r4r7/7lzoPmwEYpfBPXvHzOHvm8GTipwZxiLFoU1YIS6qm6c4G1QECUgQP1dn4UzvwlKpmAZv9yzSQDRWaK6gUkmVgO8nIrECC4M73vs6ZWUtCfY+FbajlSpIsx9DTpAy3sf53suqub9O21trQLjaG+NT5NrYHJPJa8yg3gAk8N3GuxrKPsdtrHADIqDabEZ+2OyAHJo1CMYf9VkcbxY1ot8iXTSMJE1VGMkGAmZlZnZCgIyNE42e1xOj74gpp+DAbiOwYRCbynKW+sbGFHhuW6ELiEeZmC5jJ54yCogg5UtpDnu83zm+gPD+Pn33mEk4tlPHy33kNHn/iqpuiBfy7H74VP/fiH3UkLn/Yug35l+9zo+U09VNlNh+j2JFQFAjr4JI50yraHqSEAOlIZTcdW8ESZ9W78QVC47iZd73vr90MEFeTm2ibLcZB/+kj3ukmWjfV5DQEh9JYd6Bps3o9ogBfWGvj/gtthIWiQlX6r5laFXO1kvFIeRgpJ12y5U20INN6EpJJDWn3ByjnCxpSqFCdmqhDwI1YzEUj76dGNIvzZFtNtRnQ/Le7Xck358Uy0ElIVWE1f0SYESjN1DBPn0v0a9xHKh4KeCAdhAUoYrhr67t41nXLeP71S0phPvIv9+ONb32fJk1zF2YqefzD6/9A++BP3dN9uUPVlVf6g16Vvrg0xp2aoKDGIQuWnrAxwk0w0/e2TQbwGKtP2jlliiG4+0NvSqSRhIcOaJxjaFpG5N/gAhpz5E4GDgRL0xZti8EMUeKrlQXipb/6SgzTRRx9yjOwdO1ZFCozWF2a01Ss3pB1ur5tktKiNLr9LmYrNcFZOuqQeGs2jQoHTHimQYblLOvX4MweDhvOsR7Y64l9x1Ie/SKjyZBMvWxO6ZLmE3HNkgglNbG2UCbHddRDENlmas5PCji7kMPyTA7HqkxjrA396uYufuu/vQFt+mS5oQB//cqXY36+ZsLlSop8HgMMDBTwY7uNtG2D5gSjOt/ntkxrZgefp61lwfVx2rXdgeYTa+lOhbrnI2+RmZV624DMiWk1Sfh2JMP+bdxPr6n/+nUenvObbn4jwc/+n7+HrW0jOFGinvzM78BPvvSlaGcqakujRJJqOIgiHSbDfsS5alXmlcQmTfdgi0SOvCKb8mhjwKFAqtXuKlLlzADyZ7Z299xAqpQgMObErITYUGPybGIEbIMoFdQaD27kiFURAvo8djLAjUtF3HKMZSeS1izy5Bc35bf/6A06ucgOf03hP/30j+B5z71Jm8cxqfyG/pqtG/yylMSPW3MH0MRGmNMRGHKVNmJG/SaKXxjV8udsD2GswVKDrd9kbxJnkj92+xsmeaZSDwdDec3zZ5z4qMwis283v94+ENdVxd0NUTggB7rB//jLv4Pd3bqiNcrkU59yLV79R7+NKOHh3DE2oxx2hxzWm8bFzT2sb29hrlrThuZy5vvYRENUguZX0XVEpltf0CAjYMJy/Fw15JDZNnAz0slWYFcyTanOZWFeOhCjj2ebcDOJuabYdpCMkE0C3HSkgmedmkUYM4BKaaycITUGCLz/znvxjvd8fNIFfeLwIl71ey8zDSQCxQN4xjaAyZ/yzs3x8J6EwvW3cvi/Nkga6AdRmIHj7zxUKNflyNPs0xS6xFSFsc0nPvgmLa0tPPNM/2H2AgP2fY4zPRHOm1+/6dJS1URpctJyzqmUXcMm/wMveukrUK/vq8rBrx94/q14xa+9bJKTehOzPwS+vjnAheYIVxukO2Zx/MiqiwaNdqGSmgbdG0+nP4zVbDTlLdlJSAzjWamnprAAzu+FqAhxiZChFqr9fwSwGSgmUz3GU1aK+M5TNQRkHMYeKjRclKkYN/PS2iZ+79VvU6Gc9C2u3d/82a+rfsv3GNZtY9M0w8cBBvacNnaAwY2qHy6qZX5pfGQbTadY1s2MmAZN3n8SC3ZwG1/56Tv/fuL+pibUwmFBRqpo2IbKVDjTa5GvEbsMQPDa6sAEiZTLgUjhSId44b//VTS7baTdZv7iS38KL/7JH5amaZ7QAYfO7wXED8Z4bGeIJ1pjJJmSNoQAdyrtBv+r4Yn+zWa700dxo+iDmJdZxzEPEo/UlEMMlhGlxofzFjlum/hu1AeGXYRxhBuXC/iuUzW1SNjIM2sk8vVDO/Iqkkb8j9e8E+cvrUsT+fUnv/uLmt0Xj93J89RiRa/GKuBT6iADri2jr8CGB+skF66xMard+Dorg1kgRGviOM2uRmvuyx0HzfTsnjv+3gIgfdnf1m/pAiL3G6u9TTdTP/ZHDPvCtdtUv8EePNYYthTwIz/+n9AlCcst+Ct+4xfwfc97tsukfOu5N/QWzjOQUJiQEJscYneUxqPbHVxujZGp1NRYG41TqklysZj3+bPDyOJjLkkCFI/EoJnRUU4GiAlgZ6cY05Jg0ASiAZ5zrIwbl63bzBgDju/qTp43MD+S4PDWPn7vl/CeD9yjMhUX9vu/66n4iX/zPKFPrGTIPDqc1npPbI0D1+2sGZ86XcnyR96ZVw5uJIMfDUXUmV82r5Y3x799hUtrRJd738ffoaqJ/zoI4el792Fmik1bDa36/0J9Xjt96sIPo0mkX+Mhay9+yW8YEVhnqKTwptf9d5w4ekT9JJY7kU3gYUe26VFpLXiQrfD5rsvbSBBrjYBz9QSPb7fRzRTFih8MukiHee6/NJMjs5OU8VAJwlMryKTXERZ0BcMuqkEX//ZJc8iTyBVZPkrmnspSyvECwYrEWikw/iirRrOD//4/36lmJW5WqZDGq3/vl6W1lv+5qN6dykvwXGdtO6DFb6ZtKPkn5jNlhe0/2jxfHlPeeeDUYIEJDtgPPn3n27ST01EwTnIcgiGwwAHESsJd65/xNd20qG872sgY8ErUuZHyGwnWNnfwn3/1DybBAq/zvne9XgVrmwbtvlyIbkE7fZlhm17LuUCT7/0Mae46fVOSxn951Vuwcup6rJ69HnG+ogCDo7J7TE3SWU38YgMsTzlgdDgTt/Hdp6s4UrQRAPSpHmLjsvnxLbwXDSR0f2iqycCnRr7lnR/DV751wTQlAF73x78mEpmzc5P1c/7KugUcHYbnmfiNVK1VQst5s4p8nKX0JxS5kxP/1RpM4pb7Pn6ba0+Y4ogHc0yLPKfpykHtm+7A9LspxHfgtwHwwINfx+/+0V+av0p48kCID77nLSIhs4ff2sINqPCzFQz8DewYJtfvaO185vQlXDrVx6gi/PrDV70eDzx8Dr/w0z+GN932YQS5Ag6fOYvZ1UMolUt4ytljYtiv1kIcKViw50nRVIhv9//2GX4DvRBN66ZG6fjCQ9/Em//xDrVGkGnwf//az+L4oQX5WL+Wlr7QyrpTIUI7UIApj03iMiDA4Dz+00AD6aejl+iQO1fwUFQseOXA3tx71zsm0ey3Raaug3pCH/n/yT/9Bf81uOCvR8Txwx/5FP76ze+ebObMTAn//M43CoGZ1HPcYGHV/Nyo08k9Tca8jCaAhQIzl8OSW0O/cs/nvow/fd3b8aPPfxY+fPf96HXt9SmSrYM0/vC3fxY3XH/GmnYCW1CNkDHa/bdtJktk3Dg/hnXSL+JMmwKjWN3z+K3ff53yXDYW33TdCbzsZ2zgvg9SeA/qAnCaZ+aUrsrugdZYiuJOJuJm6v3OaMl1MftlwOaQNSG5HqfldT//L+9SGGldXGzpLjpJsCW2gNROyJkgv97HuuSf2+E10tvwyYe4G3rHP34I73zPB7Q45LAuL8/jtjf/uZ0RpmaeKZ/Fm1X7fCerHn9ky7uSbyeV7l68BeHM9V/+tT/Gs55xGp+47ytotziElxdik02AP/n9X8NTzp6wBhyNIOeiuXNCnDFhdOyLywyYTFhtACQ/zqJSTjOx1INTpP72bf+Mz3/5W4iSSKzA1/zJr1tfjQgyFnVa8GIuKEzbKU7exRAJtlqxL2t5IoBppwmDnYpEV2Bqe/AUYCC4/+53GwLEX2lOm8vBXKhNn0XO58EjpExKLPrUg7r3e0b85IacNlOC/udr34o7PvEZF+TEuObEUbz1jf+vNpMzYXVWpPuy6rlLhK2leOInCb+ZwFhOKzmjTjkJpo9T42kS4xd+/Y+xtr5jqEtC9ncKv/jTP46f/nc/ZOUmHVDOL3d6w4F/8zOsaDyNGUwz7SRez5rzm37uwlW86jW3CWPm9f7uL19ha0O43h0vwusRJ+YrypUZ1XmNYkq4ZRo3iC7iDl33KeFBxM23Vk63wO3DFz/9XttjhbuUIwf42r5rsQ6aT6WPExTDL7hbEndssfdzvjTD9/ze/3gN7n/gy05KgafffAP+9FX/j6FBB6Jp+6cttBZcgDdb8ByHVL7RBjbyi4sr2os7PE5QGjUijvFnf/V2fPIzD2LEESww5t8zb3kKXv37LzeQ5MBn69vYTaB0AYbm1Lm0QlO2BkMNMeb1PePOBjDZ1yv/4h+wvbev6/7Sz/wYnvKkUxPYk4RxWh+iNtZ7YtFroGmhhv6wwmNdVtMgdIoY+d7Y/93WlQDtWVXn+/17NlKKA4iKttWx01oda0dbdOwUQadVq9OCuwOWJWHVoGGHksiAyARlEVGQRJE1BgIGULG1VoIBQwjgvhSLKFaKCyQkIeT/O8927/3++juYf/m+93vfe889y3Oecw5YlA5NYFo6B3Gw8eureTKBYFBVGl7yIa7gez023TcxxvhoPBxUllSSbkZSokVfesZHyqbN39W7B6W846A3l8MPeZt+tKOTS0uNynNUd2epYuGRAq6JRopLIe/QoQsKfoGFPr19W1n31Q1l1efXMjTZuQuo0aDsNneq3HLdxUrSeTMblUN9GSJICkGEGrHTGLpbolETAQOTsEiB1D2uvf0/y9e/+W2aq+c/7w/LksXvFRvimWfY511cK6tdNqTAf6aJONQT8audUq2BJC8hH/BoYrSuNkjueXDnV67iAWQPg2SvyQYDIK2pCop7QsNQk6f6hTZspGdoIi3VtFF9As2uglpyytnl/ge+n70s5yxbWv7mlS9vDgf3vLsuxQuBu05BHCLjjirsZVwqhGpmAMzWs0Bgl6d3lQe++8Ny8vKLyrbtsHGCFFG3cvvqTzBvWrP89o6TEMBT8ESyk5gGsHF+yPbtbMyB6/C9VWKFBaCM/4zln+Lmg8G+4sPHcfOwjur3AJaAfiZbmMXiJtNlk+nRdyC6FzoRW2UqGPDnGlBrTdsBIp9U8Bj+pQRgOMr27dTrRO45VVaMvHpqvcEo+ebvDChkSxoUMVOOX7qsfO8HD8mQj4yUq1deXPZ81kLDj3R1+L+AA8rNS83KaWoBExfD1Wag7EcT8DTDeXEvwIcf+UU58vgzypat8DrBpkD36pFy8+cv4rRauPZ9c46EHNpkAPMC1LmZ+BddOre79sVQWk/7gHZYfv7K8qvHHqcNP3/Z+8nFhTpFyg0eLKA8nsiBhhrAnVe7Oo2zSOK513DGUCU8rtNJjA8HDKEeNxVqVuQrYYXpJACTnLp7GmSP2qVzI6VWm+tipxOf1YW1GsoJPm7p8vLDH/+UP+KBbrvxSnqRvj/eJbUmwxNP46Hnos0JQxwLQm+QdEP1CRhOrcq2QhhQnPuOQ48rv3liuxYOVMzR0XLNqo+XfZ+N4TC6u6j09m/r3kxIkTNEptmhWd5tfATHwVT5smPrv7W5rPr8rbS///SWA8rr//av1W9hLtqb456V/TEw6lEj4lOpKZY+W2rVPYTc+z5hmgReK8cwLuELNjMhR1WfjN9UlEJWnYd3EhgmutQaFXFz3exXO2N7aTUQT2Px+88sD/33I3wJwp+brvskAfZGRxHAjA3mgGz3SUDJQr4Ud6nbJDIzvw+g0DR6LQzszyGLPlR++vAvFU6gAm10tJx6wlHlwP1fVQP0ZjOD8HSbyfbfOp3QVMyDMgXgNJWwTdtuUDxGy9FLziYU+Ny99yinn3Q0NxG1OOylByGclSMOMID7ULdLpO006DSxZ9SrEt3pLN0EmZt67/obmc+M40NPMi5/VWVxaDqGgTMm0q8NYqOp5jUamgKI6YhjTy2PPPIoX77Hwt3KtZ+7pKOb2LVMnQZOCzbUp5sP5LoKqKc+XuvDIN2KTo3QmlLOPu+icsd/rKdTxMT1yGg5cP9Xl9NOXKzMhj1whR2auMf2LHRqZC/xM6BJ+AZpYMhPjS0JAAAfk0lEQVQMiuNOMe/khSKbc/7HV5Uf//TnZd7keFl26lEcEDA5f6H8Emi5UGrgb7jhJFUt7hu4sJtLcuiPY1xpkOZd4z41lkQNMhiubLxzjVRxYsZOaij5Vq/Rh1wshysV+pKOqCcI32RgOCGqmVIOXby0PPror/ia5+2zV1n56QtacZJugKpFzX6n+VCRRiIlsDX0+NQbqHZJ6j419xMwH9e7+oZ15TOfu46AO8wJWPC77za3rL7mU05xNVIy7HOvcrG54idJ1eOEBqwgQYvCpkdHQwl5mIPyv7/bUU498yNlejBdlhxxUHnZS19apnbb3cXLYt1FCOFnCMZ0cbM1mk6klLE2sU8zhkzdYE3+ffOGm+VHsrRATgfiHbrEPjCSctuJjIeysSOdMQEv0Rq5/GScuacQ3vnew5awoSFu8vV/t1/50JJjKrbYhEkqloAAUkpIAIwj9JhgQQ05Roa9/p+q6ibncqHcomX9hnvLWedcyCb2uCc4X6gRWXfjFWraa2RJAEJ4OopzmR+lA6RwpI/ptCayWWIsOv8Lr3R0rCw69jT2Gnj1q/68HHboO8vcBbszhYeTK85xvFYtpMIObZyKnCVk0TAJSwL86+88yxXeG9z3zbX8FXrPIWPPxvCda9yMrtjZ5MGmAreeCg1uY7THtJlsJ+ybPq6Ug99zdPn147/h3z/4/kXlzX9/gGC0CIk3UYngnTwFlCZGRRobwUHnRJz88F16To6TpdcliTjZP37oZ+X4pWeVLVu2qlQAzSPGJsra6z5VpiZT34F0mxhzCYewcQEH0BotqjcqXOQ1CS1VITWQHcNBKavXfr3c8ZV/L3vvubB85NxTy7x5uwlssauP9waQEIynTeV6wNywqLmx1rVMGrqaXGYPKLAP373roWYxz8RTVIlG6KI8nR5YirAF2GDt4OWNVPgwzNbrPVvVLJZy0LsWlS1b1J3qqs9cWPbZey9VHVfEBw+A3Cds5TTDHGgI9CqPPZGMxHVTMNN/hY7Ihv0cEfEM4bNDF51YfvvbJ9i6Bu+HQK694YqyYO6kw58W94jmoROJ5yBpmQ3t8zvZuaFNhfCbXMYqs13TZduO6XL8B05lx83LP72CHbFzAtPNpYHd/VPoVAYs6E8gT38cTOd+JWTY4FGo2bUUBgmMlydQV79h2Ex6V5bI0BWS5faHcB6mT2S8RDz8W99+OLtk4OtLt1wF/EOhicvpIf0AKuSNjjATj+w7oS5TWGgOfO3EWZLO5vFGsDDFKP3Oj/rAmeVnj/xCADVY+6NjZdnpJ5S/fNmLq2mhGvX8kfRxYKzpvrOMjw2EJ89IoXeZYU4OUlwIi57a8XT54Y8fZq+jl/zZi9zmxT0FepSs8zV0shO0yBZnM+Wdq1AoBy2ReQRv8MA9X7Tn4o7PAl913P0XvFg8FSVOkwCtrIBOUq1hK76In0HZeMvB7yvPuGH8ujVXUuJB7CIQPYPpAsj8K55EfhOUS53I4dMnyVRAGrvVTIGeAQKBIlZlOqbL+R+7oty5YSNLEXDP6NP3joPfUt7z9n+UCLsEnTNHOFldNrKNbJZ3my+GRy42giPGw2DghMbG/COyETjiWVCe2r8qpJph9sTraS8q1Bwdq/ZVTVHnred+IADspII72vgNYLMBepunlUvVhvo+uVxEg+35wP5Bq+Pkc44b2bpjZ3nbu48k7xS5wXVrVgnZgYogVAZPE6oCQDPQEBGAuXFO6DUcUi5e9Z3thOD2+GAGNXDSA0KsvvH2ct0X1rHQB/cDxOrFL3pBWXHu6XXVakhFdvwz5sIKzosHW4XGEB1LDVxPEu+dvB3OGhGKxD6DjI2birQEDanMCKhSlQ4F4+SYLsOT65Si1sYV1KFrbvrGGp5temUu3ORJJIWhEZ2l3lo1U41FrV4jmTk5lhXe969+/bvy3kOPJcVx3vypsubqy4F6skwAoyLILEDcND7J1mJVnfHdAQcd0MfLq/RHkb6YkiKpCuUEqKSSBcXZuPe+B8uKj32GM6jpWIyUMn/u3HLDVZfYAfOpS7bEnnCgxCGL5nWwP8LNZMm61wF2GQG/VF9YjQHKTVa29uvtX8IifZZAiFB5+iwVnkoNEUOnUWET33XfnTf6sU0/sIcYej0uBAmUa2y4zwh/KPZUy3SpBR5H3HOzDz38i3LsktNIcnrFy19Slp/xoYJS9Z3btqg7B6qdJybL+DimxEqINE1eJ5PqFNsSSj8x2MYLkqOik8ByOpYL2rmCMD32ePngyeewWCjwF4pyv/iFy+UlBFZ05Tdyn7T3rp2s6rWqOYPlzG60agCqa6fq6qZUUyWV2yeU4wDFNOA5ND1IczUBznPduQfJuYJrq7gzjiZxa5zOzetvIjuPx9cnETcCshJ+x2JRs/FiWwJltYd0esYAQ38dbPD3fvBfZekpyzlq4ojD3lne+uY3lB3bt7AdG9TSxBSaMKBKzF0k2KNQqR84TyEd5wHAFBehON6tHoyAPIbPsFOyKKPhFR2z5KzyyKO/MuN9pswZnyxfXH2ZVbO6hijOw4lSTMnT3YEpGjXsbivRhv1J5WZLoBKWtVPtMK16qviL9VdX96qMjVjzAQrk8ACwMBZgDUvTQoDFrItsZhwBOiymSuCmpHKFh/Ir+sXE6NnhQYRC51PHf9MD3y3Lz/4YsxAXnHtKAY3/6afhoIxywvrYBCbOKVYNDIiAm2rSjpjMSFvcUEDjMeMkslxvu7pYqTJNpxt5zAsu+my5e9ODdIJwElGredO1F1H1MylMeEyLg8Q2VTdyqPERSJYT5TIpwVRk0Y/g7TUgAXzXpjJnw4w9608CJC3mONMpuIQyem5djaBB17E7760nM9ARXpwp4zXOjBudoLxmwfFQzdXu3S8qhvTBmZkpd92zqXzk/EsLKjZuWHlBmXFL66l5uxGmw41q+jnojJpGRwSHp8/OQJCfJGnjTdafxenBq7mRNUepkvGrrr253LD2yxrMjWrnsZFy5cUfLs/e59lVSBAqseIbjSAcV7JMgP3xOHDEk+0HZRRV2HbWspmKAGwWbEMD2yF2DXqTtem98oaiyr4GVJCM6KQm7GI3I/9Oh1DmjSkwqk9nGibArPYJgGRWpK5DVxJMI5UlI2kQMTqlo5ZAwr/6tfXlkstWMSa76tJl9Ggn5+zGZgzoawCoLTQMuu0UwdS6hA7p9iieQYbTxVkrBjnwJnbnNLksNaN0FwalbLz3gXLuistZ64mC3KmxsXL60mPKa1/zioqsIN0mIYbNFAJFNW12P+5X68GWLEosMxXonoKkiUoVYw1ZE8P8cN6mnHGn4ggwhOcT0D8aSJvfTmUEQuGPHEJdm06LCV2DERbdcG60SV10//saknoyjA6Fbeb6+wrx+XV8r/NwN91ye7nyc6spiJetOLWMzV1Qpgfj5WnQBvFku1TQGmI1kR+XrEViZ5caVvQofXDdsAGGJSpJ+VLYrwEnDSw+7ozyuye3svyPk4He9Ppy9OJ316wP2uXodjSgtX6lS9mI2merEJjdDx2PB3vCmrYI8amntqqRZMII27icNh6innNl3rDWDiV8rXgoIAkuhTystJaplrHrANrzZuKLfhHWQfGWu2Kgq0mXvMZ7ghEm2A06wwWBA+HY6s677ikrLlxZJuaMlDNOOaHMmz+XTsoUZm+OjrEhoaBC5Ck1T6XPrfL+HM9VJmFQn5rgdnsVG/bEvoo1AQaMlEXHnVwe/sX/1DmZf/z8fctlF39YGDHL8NQFGvCdOlOLXoqFZek9eLYQMpff0aO2GsQ9M2VlPhDgyJ2ceiCh7oGYoDh4M70Ez4+Bx8okA3KWTojTKXOIg5SbFIMTITaBOgSDMth01006WwPR6RMWaIwUHkZqIJ6jglXJbDYzniRDGBeiRqfD5mBj0fH/sccfL8/e61llzpz5fEBQH/G6Flca3fGAmnY0Wopu6D5oMBIjxlvUaZQtSfCtxg9nfvjjZcPGzWovMxiU3RfML2uuv0wNK5zPxIbihBIBqn6CEtGIgVW5JYdQSBA/qL/V6vegQ6aA+HY/8Y5lX0OO0UkjtAn1icJiOHOoO3UFGdkKGIRQSxj0mcnkUNluuutmjlzMh/RoDq0hJVthS1W7Vhs05Mx5ClDgSAh/pbSOJzQn1UKQkCfBMDMuZCwkVm2fx7WCujYNMoNxwlCom+Z0RFJL9JuiHnWRsnLV9eXaG28jCI+vufPnlNvWrKzjg5FD3TWN5hbKW1bUiTnUMOlUqIuvdBBhWNNtKtcS+U6PB3FapXr3od00YZHPEpGgE4bRVeiysusZghLQYOjRrqFvyrKQVRkiNh5x03qlwKjHpczr96yZNPNgqFVMupDU93g2FeiMnqUZoRiC/GqoI1vQvDobcT8Q46tZdEP0WRfKIydl9hcYCDkSFLxAjp1Xefe3Npfl511Ytj2F2dMzZWJqrNxxy9X16VnhhSGnLqZVkTL+TwwB0CJ9xryZwbC7rFFOaYfzyncIDGkaKaq8wWLgVMCpWoaQUEvq2vwn86MGqEnl4QrDz3tlfIUns8f5hhgDuTEvXnrWZCHjduNnSYmAhhqWWDiQ0gKygaaKMOpotcmiGfJ9UjXWOEAVdHCHq2CbUe9DIIc7gbEZkh2uvI62yQE4vD20ajv0yJPK7554kuoPbchvu/nzHBGF0l6oWJxOshzwsATDR81ymCgzI9YglRYpL7b6p2EJsPeg1Cu4QNIQKvpB9CxBb+EH/Q+C/aYtWPNlcBvRLc4C0ye1NZMzyjZtEJcH77lVBzILb4MuaKrLdhO7deVufY0TZ9706Rk5SzraxkadfYCbjtZnPVCs1m7JlDsY50MaJ2aE4pyqVb0u3TxlOCsURrP24oSlzRlDB8SurKp+phz9geUc1ahM0Ei5/NLzyp/s+7yCe9+5fVvZvm2r70nsAdJBMEVigEl8hjQJOQ4DAdSynbqAeVLZ3w47UdIchEJmCQCbUs3KVSbprfSeIJ9dM+In8bOMAjWEqpTBA3ffTktcrV3lmghqoiPD5ojq4RZ9ELqgHB09BeIz/tulxHgzsIVpQAyPjYF10kaS0lxb0/lUO0J3nA12R4jKJJBOPIbF2sE5JdA84+zuBWoGOpLUGJFtR0GClio856OXlXvu+zY3Fx7gCe9fVA583X5sFwNbirFSWSABBuC5mnXu8AdCjXvSDJKW/oppUNynOBmThXRSJPjxD8JT17p59W17BeL0vSWEiePzZI8lSDz7/BwnUL6z8SsMTWrpWAdg4y44+oIhhjZtCPXpJFHi4g/zyeQNGTusgTddbTUzlP73zTCu0+s5prC3qU7aJvbNx8I52LF9G8siAAsmbIEdol9MvMAdlvk50+Xq628t133hNgb00IYHvu415UNLFnMztzyBERTbJBxsjjxWBmzX4nQcW31aqIOn/h5PlgJoAUe5hGJWpcGqVkkJXx5mFmLUHFJg47KV2jx4u9oTlvy7+JnLv/mbt7KnAaWMPUJz5MON7WVICz77q3m5bTNpB3rB6FAh9XzTJjb8UVdNoM/NsPvumMn9DaTCFZNhzrMlu9Y7asF79awLC9f80U8eKktPObeWGbz4hX9UPv7RM8r0LnS43Cqb6Rh6bGKS9hIV1zp17mIWWmTnLPIzOmBenCI9A3LCVcBIIwXZLQTu0G4SRmUdBNrHDIXMxkehoIjVn5+J0d531zo6QJyeqtq3yhSjcqhAgi4e4nGcHyETuoEZ28yA8tlM/o3T3pUnDbbod3kTFUtkM6mmIjgOP6Xy82F6N9QyYy3bzKSMaijVCx/qUKcH5eB3LmJrNtzVPnvtUVZdfgH7AD219cmagYCjNjoxpdNpFjrrRqClsJk109REWybH/zmTwfCkNhNGmKHYE9cQwz0NOVwWEniUl02DDm08sjYMvXJI4mza1A02rb9FhC7uSIJbbFCT0JoeI2CvUm2EKqJUpme440FfpwbHfla8r49n42BlKXIa+Ag1Ae0hrdSvERh1hpS6s5ag/ZVzFtQJjkJqH5t3DXMyWg478oTy0M9+TjW8xx8sLNdfdSHTcdu2oE+uCj45/WAcXaWn2M6lTx6w3HsI6mz2Ldl/lDEwE1RL7hq6pjpYpehk/2V2ZnNjpbla7K5io8ZYaKCIw7yczLaoVqvs0e6jXz3IeKmudegksZYsdCcnp4Nut0OEqh7dBJ8ikIIjp9kCG9bgGi4YPovXUJwZAaNwEXoLxCVTALUTJmEfQsEPOe1fV5R7Nt3Pe1owZ6qsufZSzgDDPBVuJkZtTM2hUzXKCe3usJIZKV2rM2mCCJpPZTURCkN4TJiLHG5Rl1MM7ZZmVBTIWj1tU5QKgWmV+w3H2VJblMH7N9ym8gQAuO6kRdvZoTmUwgrudtBUktlm2PXwWWJFLrbtcFRkNkA2sZGw6AxZhVhvCzaLLfK/1ArpfOKNxbTXIEpR61mYGgrY5N+09kvlkyuvZXw2OToo16y8qEyOospru8GaEatYjWtObx42hHAfgsR+Mi96MuKonspUp/t4o+up65jp1QvtYMf+5GGTwJ3lc/BztBbZ0Kw3B/BgHRCacHyU0RW8UbQF2SdpTVUqM0hxL4DQH2cnp7lBdnYEJCgLTvtm+xu+0dCJkfzSnqgXgNqkZLF0EkU6biTgBnRXwrWzHXpQT8/r2pHj9488+lg58rilZdu2nZy0u+Kck8sLnrsnPWN8AQOFvUQ9ZeAzaQmvQXKsrt/MoJgk81Uj0oqr9AzSeBC5sB/SaIKesyum2/cSyQwP4vMYstS6Rf1isV2m8MDdOpkhVWnZpaaiy7GZMOREcZDRZ5X0mApsQ4IyoMw2ZuyBM9xFKpmVnuKP19LLMy7LT06JQ3hGVK/ysMX8k82ocGGYaxHfPnVlrxd/omA4voWqfdt7jy9PPPEkTcnhh/xzOeC1L2ejp8H4eJmYmC+eK1q1VE/Cwsj7E3td1dPYKDhFcuAkqC7kibrsCFjp3hJVGYGW8BnfTo7Sn62NTL+/9PFtFFE2nmyhSW+AKzzLzUPgzOyGe8jp1Mk7rclrAwDKmlgtcJyxCNG8mWpYhIwoS99WikGwy96zeXV/YncsOEkpWXa5IUwPOV8UOybV51iXDIRM8pkp7zvqpPLoLx+j8B/w2r8qi//lLZpzNj5JThIIZvBe6YlGYH26gKoRAEQym4fCZRPd5sVjEyjfHEvUt0j9+9iYJZAQDY0X2wYPr0/vVNbvMzoK17x/w60cH4WFlApVBiTjFivHxouizDoAYDUdxImlCmXcBLUqLxgwWPVQzd7jIqMRhpl+BA6yI1bFcWwYK4J2z4lzVVMz1mv99IyEJElLwy/EqM/+RK3HdgKUP23ZeWXzt3/Ce/zTF+5Tlp10BFn2Y+Nzyuic+VXFE9h32MZGS4Nx91mHR924POIvge6iQB7XVUMKQYAhPEflpl2NNjZrIuQnQhwtlNdkFeJr9F2g+ZoH77m9Okft6LfFE+VRl8+JAUEqYDH+ggprqt4xSLJUYtCYdJCMBxoVqeyKwhk94NCOVRvOQ00YrXFQYzOIqJhaESeLNsm7TxOQOSJGkfTeUm65/Wvlis+uZt5w3+fsUc4761h2WpmYml/GpubxnlgOQKIzEtcAKdDvFgO+UeaHIRwKo5iwtl3Os+Nv2kh3FXFsiusojddi9thLoYAG8wNIdCzErGGuEQdIGnqkDL6z8ctD65gfmg3VIqfQk50w7JEB88SmCBpTVp6MNjfuJ4DcldfHw8Vp1gnt8EraWNsax48YY6Heq13iuav2kjqVrmbo4/J8giMGtKukdyoQYcwvH/ttOfyYE7kxu+++oFz60Q+W8ZEJFsUi5QUhfPppIVqY9EPeKjtVowCoNW6kQ2ZojtBaPEs3jaD52IUxWs5F9lgubaGT6J61kriS2sRcoirwMWH+l6hd14FlcN9dqDVRaJJFa3wTHX85Oc170g2quQM30k0WkoLKXA9ubJ99caActkBUeIcJ0GALNFCf1swDGXbjW9qpF4hgtwH3haBIGIlcRQvgu7GJctC7FnOc1OTESFn1ibOY1Rmbu1DjlHfu5KBysvScgoLpQHMrQWxuB4AWseyh5OFxSRCYDNejWHUt6ZWrwqzZU7eDMU1HJslkMMfS9IYzrMYs/pQD8tQizozbLKJtwxS5CMxotBylYjlJZjLucW5EfXCKysU4lReEU2vVE4XKG+BxVqZFuLsDbSBQfmjykDxlB8cg6oaFvlU9Jyng0RI1kb1LpGhtgVqHghFeSjnkyBM5SRbnftnJi8oee+5ZRiYxV9s9Zgk8GHYbDMokWPce2k3VSuuTcTJ2thIOuTsLNyUaxL5DA0Pw/r6o1nh21zQjfoaiw/ZafHScqdhUnswsTg/rxaOidneSV+C1Im/dpIBnOTGOE9OF0b2FqjUXpVSLOtS8wiUIWW4LQ7pcsugVFMoBqIsYKjrJijS56/pYago3OMr12VGSvdTVbEpAg3qg5z2nnHl++d4Pf8SL7PfKvyj7H7h/GZ+cqszAuWjwOznJcY5gD07NmVJBU0KGKuh2K7yBdFxqrz/ZfKFX8T8UKrWNVnQQx6YC9lZHgRir5mtguHyZ9H6AN9ukuwWjCRUQ91Vko6NbhioflawAf7hOMm5UYi+iJ7EDLh0Xv7W579wgxpVmIaBUYifGXDwllT42zmb7WlTcbyBHhAkuUzD/FYuCKbiMo51cF6IkH+DmdXeUz16zmk7ba/Z7RfmHN76BwjkHG4iRGRMaQj5hxvvElE64vmSa5HwKaiT40nmm0jztK4eGIZ292Hj3ShCpAk1yLf1Vwytcq6sYpx6LvfVrB/dtWDeDh+HEdccJ2XghLQK1dTr1n37f2SKDDvl4bJhOrN6bG89jSULdftNBd/ubsVdnWXCqOBrRQ82hJWnb6WSpF1G0hZbYWXjPpjaCl5uoZgC/2LrtmXLJJ68sW7btKG964+vLc/beo8xfsKBMeho7Yr5IPl4/Z568XGGhScrjNUpSB2CAP8ExT+kl2G2o9kmIGhEyqxc8J+XSlWw5hclK8eR2IZ7W1I0rMt5r892ijYCnGdUKQ98gN2OPhvXi6kdFVCcGF0kWoKrKndwEcWhbpiGErZxjxH1aHC1HBIeYcNSTFwE5RszPTFlb4uM06q39cQFxWZBw3YRI/bry97tmyk7SPcGOTz1NzIhezaoVDMiZg+lG7Qo5lTl+NYdpU6I4UKc2taPVu07iwNIXu8rZ0z1dx122uT728nPClXLEeGed6sGDG788o4a0SccoPFCT1nSv0sMmruED2qui1+n6SiYcPEMZnhub0nOhGuQRhgEWLqmsqIwQmrhedqZ0rMVwwOvHJyfLnDlzh+JSfEYY752GMoDhHgU7hRGH3BzB7e0YQha931VVFs6w2yfBW/UAWPkXSh6HCpJrZru5pia0yxNVjMt1BB/ZQlLJ004a9BXp3MRUshu4CbWzYueesjl4cOOXZtB5isQlA+4KGOV+p4xOqiUqpmmt1rRPVca5WdyEmhMhj2nV0uGq4Omk2jinJukiPCxmYJM/mtZrLshZsHDhkFBF4OBbCjhoJ0cbZbuVheo8S3yO+qyD8KXaEmU3mrOiPnw6sZgtJmfEvFl/XtJyUaHcAEsVMh1JGIRZQflU5t4C1jk/FAD1i8+JV4gS38DJhqEkhJPW37//32aiqmrOkWV8GoCiI43WpcPqhZtl1nfsZ15Rpxa5h3hNQfkBsSCsoxiilVjSPd8ES8tGSumXY6L1/AW7NbbBUO2GlfaswpwE8VTZvkEx9loIVjWOjko1wZlxSQyWczJRaxIvFFqoZXUSo/dqnI9bE+jhPcXeCkumxQXdtAqj/s55JmngbGwbJkfnTFRVaa0mvYPvbAKhq1H39GC6oDbZCdKuZ3o2GL3oshAVkrKK1PulZsUIaNVceeBI7+zcIIeadoCs1FBhM6QJd4xuNlZXk+Ch8NRuWASx9t2R04E7iT+QZ6w2r0JofW/XeHDm7vjmU79JzJWNolRUFPSLqTO81X9P+qp+dgTdqhZcBvkKqktVxqqdoBxU4t+pY62dqw0dYjMD1fVoRDDMqv9r0rh5cthMLiTL2JySsfGu6ZxZeclkIOgsdBSInJx2atz5mS20p+mkzJsLANxkMEqlsN0A7xScToPEpg1JMD3JNnUgmK68YifCk+XoWtL0oUIEaUigwutNqX5FnhTeBL7kNEWXdOBWR8lAUPNGdDlJHUst0uLZSnMssy2IV6eYF93VHOp8b7PUbG+8A51VVUSMtaXG6ul2+xM2YepK0vE+JpjdJLZeJ1rB4UXtDmIV2BAkZyNadE422xQAcNUdVBWkWn97wQCxO28Q96kpEmaLW81nrjYbNtnRymb2ahJsp/BX46zEHlJwKhhn7WAvNqoOlnPUNZ0xZVh43E8PmWpzZffGxzHnxUBMvRlptuq0zZoDk1fTm82pijcaRycWmDfHRUvdf+xNU3E5yRKELhTpu0bHxnVs99gMAvJJ/6TqOvEccMwBNhO4qFNESVDXId2NEKzydR1dZXLUODiqXuUHnnzUjV+uoYzDiYQkOey1tVrnyEVV954+ZSbxuMEBw07WvBBIXTVt3MJ6bIyDah+qBsMz8e8urVQ2ScLN776z6Q5RLR3jKV5rtpU2052xqkfVEbl6SZbagTTrRvvX5+fZ16iLYPA+TlEgRB2mmTKOoeOct9zSZVVSmTFpoZTAjah+JqqGuniZgFJrUxQHKkuhEYaNuoJnh6OXqjNlM8w47yYQsdSut3FxuGJHZ8XL8CeSbUqRcTuxErw+fFIcagzbIH+yUIlR/w8zhPQ5IIcBxgAAAABJRU5ErkJggg=="/>
+        <xdr:cNvPr id="1036" name="AutoShape 12" descr="data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAHMAAACaCAYAAACaCHesAAAgAElEQVR4Xny9CbhtV1klOtZeu29P39w+t8lNSCCBAELABkVsS0osy6KeInZYr6TsyifvqaWWlPLQUgEFFAGBiFCChD4hICGQAAmBELpAcnNzu3NPf87u+7VWfWP8c+598H3fO3Bzzz1n77XXmvNvxz/+fwaPPPzxJBqPEYYZpFIh0pk04ihGJpNGEKSQJDGSJEEcxwjDEHFs3/P3QErv4e+DAEjiBOPxGIPhQD/jv8N0iHQ6rfeOxxEymQwCAPwPr8PP4HtTQQrD0RBJgm+7Fv+RSvFPyq7dH+havGYCu0YYphDYVRHbX7rGaDRCLpdHFEX6w/fxZ3qv7jnQz3ltfg8kGAx4D3zGCJl0Tp+ZINY1+Tr/Pj2fuwbfy9/xWnyfPUOge+P7o2iMdDqj3/F5eb9ci3w+h+FwpPfyD38fJ5GeJU7iyTMNh0OtG6/Hx+Tvdd9Bovfpi/dy/pF7En5wEPBBx8hms3pgfvFDuXn84gXz+bw2l9/bDae0CfxgLpDfNLs6r28P7L+PxhFCLWSs90VxNFkkLcY4soePI4SpEJ1uR4vAxaDQ8D55DzEXjddIhdP7jGKMozFXXBvJR+a1phtn92sCBG2avy93t5PP4D1r08OMpCIMtVa2mBIUW0zeF3/Ohebr+bNsNqON4mt6vd5E0HkvYUihNoHIZLK6D/7MC5rfTH4OFUF7kA7R6XT0GVwTL3x81iQaS4Qz2az+Di586z69izc1GPQlybyolzTeJDeUF+NGD4djp7UUAPvjN8Y0lhLETbQHp/poU5FIooajkTQkFYbo9XvaGP48HYZ6Db/44LQOlWpVCzgaDfXQXmO8gJhGcJOBMRfACQ41mRvHReB7vUDyc/nHhCInQfGbYJoJLVaAFAbDoe6JCxXHFCbTtCgyC8Xn46bx/XzveGxWgK/jz7l+3DgKFd/n19MLGteY1/LaTgXzwqJ7cGvL9ex2u5P7poBzvbhWuWxOlrTf6Upog/OPfIY6pptrNpsoFkv6BS+cTvPBzQTx96blAYIU/21mihvJ1Uz4oHFkF5XNBeKEZndkmxObKebN8zW6YSfyvGbKLSavS3NL7S/kC0iFNF92L4PBwLQtTMvcyDRFMdqdDvpDM7+FQmFitngfppncaC6WmVv+4cKbEFNYaIn8a3mfoYSMVsQ2eIS9vT23QSYQ/MMvb6LNcuWca5paI2/uKYz88hvGBaIl9CY2nU7JsvA649EY+UJ+qgjOzXHdtRfO1fHfw8EQGd1LgOCxr3064S/5Iqo0FyubyWqxuCFcTJM88wcmlXw97bxdnO9pt9v6kEw2Y9eS/6VpSCFxPk/SIHs/xohmR4tFLTYfJ42OaGJimdhSqYyApj6KpNH9fk+b5U2bTB7NEf2INp33aM/iTaEJovl50w7zX1MTTE1LT1wLBXo0oj8KTDDc8/I5wrSZSD63dyG8FwkgNTkdynzyM7S4Ad0TBcXMKv/mug2HA1mNfr8vQS0Wi+Y+5HbMQtAK2ueY3+W98774Wfwc/ozXpwL5ZwzOff0zCV9IqacU84uSzzfxDQpYnNbQLHoTUC6X9T0Xxj7IfJB3yLweF0PSaAYXiYIQ05Rer49Uhs7I3sMbl0nixg0GbkNS2iTvu3lPdp8hsllqATDqD2VyErdpFuCYb/GfxeuarzLN6HY7zu9zYTLI5bjQ9hpZIjAOSLShZuZHztxasOIDHK9p/D2fv1yu6D3jyMwv74EbR0XgtXk/3DQfbPE6fI1ZCAtmvOWQVeRmxrEsFfeE1+GXabkJFdeD19Q+Pf6NexPvcOkfer2uboQmgDdQKBTdw5qmcgVNiyyIoeSadvk/tnH0v5RGi4BdxMmgJ4owHo0wGA3R6ZqtL5dLk6iYi0JJnX6ZpPKe+LCUaEow78v7MdO8ZBIl+qjVTKAFLGZJLPKjMFm0aeaQGiItDwJpRBwlk0Ajiil4Hf3ca7zfGAVyqRSazZauwQU1y2ELzUX3wsDrU3v9z3kNaqWPgKnNuXwOSWzBlRc+c3WB9oMBVS6X0xpQ0SqViq4ZhoF8Z/DwA3cmvCg3xC8QN40PwYWgD+Xv9JoDgYxCZ4XZIZja8N9eyjLpjMyk+VdLbyj5TGe4wfSjCoLkO2kuaE5sMbkoJr1a3olV8A9Ns8XN9oFDr9uVCeai5WjiXUBkizfStfxrFS06321xggkgBc8icTO31EwJgrNYrVZDC8gvbhY/v1qtTqyXszsTzfdmkMEZN4/3YfdvQZpZQBNAajLXOpMxa9Lt9hW7+NdRiEolPi9NqykZN5TXUNqkfZA6Ifjmw3criKQqm902+xxFlnNx9xUkDEeSPMoyzRJfQ0nhzxXKO7vOIIAm0G8SAxRti+y/02gXbSLlpdD8MP94gfCmNxkz8GKQ07bXBAFqtZrMC1+TTWdkivhF/+Fz20jCZdG1N4cTbU/MfJqgJej3u1qoVquthcpm88hlzarIslDz6VLcgnvhsPs1YTSfbEGa1yqfetDaUfD5GfybAsMN81E3N4zr7PN3bphZFMutzRKaMDCu4ecyJvGxgA9Gg2889C8umjWJGY/N9zHH4sJy8xh4MGoqlopaHGqrJMIyWHudAgFz1tS+DLWOKQ6BB2eG+RC6CZfUMwCiRvPmuSg+1OfDUWCUi7lN5oNIss1QTh7U/LtpvoRKaUyofJP3Yj6Gpp7+i5I9Ai2HfG5qmhLZM9h1qJlesLK5nNNW6ZJF8AcEk5bEm28fDHIdJejOf3NT+Dw+0vfpnpl8D8IYKOBz16nb4hPbU0+sFRMImHD4VEsb+q2HPyXjyYWks6ZkUzppv7mo+kAXMSrQockQOkIttdzRm1yLxuz1inqRyHFTa71j1yKNzT9I8pnrjc0f2kKZWfaSnAnTQn0k/c5HKVXR9ZmTjvR59N38fG4go2CmKjSN3kRZsGb+x/tKftbUVE0BBSQENMwfKkUJQ5nyVMoib37xd/RX3DRLM0aoVKpuw0zALcWz3ynpd8iP37BppG3BmlkQi2jtvmwjPbBAwel02hP/LRQugLKPyWb6nImLxQ/nAjHHY5pBE6MkVT400MKbfzKoS4iOIQMTH0LTyofl+/mw9iBpXYPX85tl18linMRKYQyd8f7Tgp58Lqe8i++zfNCiPgMmHEriIkUTX/PvvCdL8E3LJkLmoDyfmvC6foem17Tn9QGHCaOBJT6o8lGth++40KZ9mQlg4t2KaZDLrV3axPvxG2baadaNz0gBlD91AZvXSMskKCgGXNCKKrrPpGXxgke/ck/CZNXnhny1jz7lb4RojBFxQembEoOYuMCTJD3jAgenwT7SlQ/T5lGSTSP4t/yis7XccH7LzeQ1+eBeY7S4boOFxPB9gtIMduQbLXznTbnUxiFGBkxMERbvZ8YR4ci+Q7kMyaHJpZYhCUCzKsFyqYmi74gBDD8z557HhM4HjnwN4wveEzfcfm7xgTejtHbedJuZtaDTa6R/vaFvhj3zM70QmABbkMkN5d7QFyvyZapGl/To1z6d0JdwEU16TTsZZeWZNCsRZvLvFoubE1kE5QMBS9hj3v0BkxzqGgysfF6khREaRE00M8xFGdLsMuBwOK9fKN6k1yj6Qm/afU7mTbEPUpQ6uBRAGk7fn04LmjPtJJjBKHUaJfNefD6dJA6eTFFrfHpglqTbtbTAIzhmzczfeVPqcVmvaR5U5+95H5aaTFMkPhNfY6mIpXDeYngT7N2P+UxTBB8/7Oxsa28obNLMhx+8K/F5Fy+c5iLLHMa6+ciZKN6oRzuopQYm6COQyZnzjscR+r2+YCltNNMAt3CUHP5cyIZAdpNMbbByViUyAgzo/yhEftOk3c4HcYf4wAb2J0KZ7DbMNFqwxU2kMNlCMQLmffivgxtiObWlMB5ODlLTAIvPKYhtPFZw5asX3iRzjaYVJg/jOYVwgZLPkQ9upqFEtn707byO/+LrvHX0a+6BBn6+Lzp4rfcZSPCVL348kaOW6Zv6I29WLIS3ZNpLh8BxVUwsR4Lg2RRiYo3cCKcVVvIxnNb7V5/Es0LiTTpNOTeC/pHX401y471Eq2qSOFjO4aweyOeG+YU46PMPSjpTEGo5fbmZKsNqiYPL7I4Glv8SxnMax2ctlQqKtPnlo0ZvOg2rNrDdozoeAPca60F2r3kK1lwAxQ3jJvPv+fl5l2oZOMA187mox80VfI5cFYiCycBK6SC/t8Az+OqXPpEo8tQDmo/pdXvaQCX2gQUyXHw6Wh85Ka1wpSjqg0zeYKhFM/B96jPk7N1GS2NSBmT7wuZwPLQaqqtREg8+CMFJIAQuW6XBJ9weFqxWKw7YN1SKD8n3eP/Ff6vGyo2kho0jZHN5c7MMPpwPcumqRcoU7HAaP/hgZoIhH8iLLeUwKNB8nsFs3KyDcBvXgRt70NS64EFrbzm2WRAftPl80/tbBUXOynjMlpspl/W5T78/EaLgCr6UYkmiq454FEcP7aJRvtZrlddCpZzUQNb0WAZz+aMvFzGloQCYLzDtU/GbIHTWQmsFOw6CU8AShhj0Bsjls0qJ6Bd4fROO0QRd4uv6/YECAvpnasDS0rIKvSa9VnD3PofXbrZamKlZok6AhIvkTTa1c8SAyGV4/r4UGces6hgWy9KUaRHx3Zwsi6J/V6j3AuHNrC8q+GDGgw0H82OP13oXI6AmiSUU3cHASoZuj/h5Ch5d7CEz6x1qsWjAuKWk9iVJYPTu3mC2PC35IfDO8H1hYdHCe2m8h9UNEtTGyXcaTmqbaFWYSdToAp2DyIovv9Fi8AH6gwFazaahJFnDQJke8bo+ifdwo1X3LS3R3fjsg26BQAKDroEJiXzh0CLzyWYSxmMOSezY+eSykDCiRX0Fax6nld9y6Q0FTeC8y6UpFOm0Rb0+mjfEaJqGeT9pEKAVvL2PpgXzRQC5O1ksW8Nev4+CB+1d1hA8/ODHEitvxQbdOcn3dI5Wq6UP5+JxcQwlMrTE7HogLWHk62E/vUbmxHJG0yIzH75WSnMorQ24GMRRBxMzI0y4UNImCjUS3WMoE6oa3pD4KVAQIO9LXhbsqJLigA2jolgu7DfL+7xGvW4luISYdEGaWuQz0no4jeR9q7AgONLhtUw5nJUCn8EJKK/Le83l844qEul6Ucx0y/JUj0AdhCw9O8OjVL4y4tfJR7XSXtaLXR212+vp+lI9F6kH99793mRubg7tdkcPlabvi8bIi3HgTJPyS0aO5hv4veWmKaddzNVYxzOh8ILgE2vjsFho7tMTFocZIUubXSnIJ+SSdppFZxm85bDc1DaLKQ/B7ilc6GkqFt7zPd1OTwHNzMyMQH1dxxWdbYEtDzaNpiuyIMtWKJCpNWTJknRfeKULocXwG6/0yvlHBXqhUT1mZ2cnmukZCcSuD5pSA0Is7bBCufl7Dxh4QZbPdrCe3IyLC7TmjAkGQwSPfOXuxCTaad3QElouvnwWXyQgwSA8zzJQWkBUx6UX9Fm+pkk7z9cSsvMcHl7Ta5aPZKlVSo4dKE5TY4SxSJtJn0BfYeCAmWkvDJ1OV5V93iMFSYGZy/s8xKho0hWPhZg4/DebDjF0uKZ5B/KHFJQjBteCFQw9GcZxgA4rGeMUdnp9bDY62Kh3sbPXRKvfBbPN55w+jOc86TDKmYLez5yU92QRsKVfFGQ+i6+2eAGdQnseQ/a5qwmQ1V4NmJ9fXJi4KUPVQssmfDHj61/+ZOLzH0WzKjtZVCYESP6Si2i8HJpPbgBvloGBoCTV7SxKMzNmGKMiYQVDVnWYSL/XApkvSw8oCMZgc5rlsElek6U549P4CHmqhT5KUeTNao+rnPA6up6LICU0FBSlJxHGCdAfDTEYkvE3RD9K0BlEGIdpXN1rYm8YYbvRxCDJYoQUZmfnUMmFaLRbaLOalC8gmwoxHPTwxBOXsJQe4zd+/Ll6Xp8nWoASy896CNObTwNpjPTFn1n+aJUo/tu/zueSsjYqUxa8gbIypYr+rjL15S/cmRysWmTTVg3nFnpyFj9EVBJXJBYQQF9JuOkAkiPtm9AWXbBDmojjBknrCH0NBxZcOX4RzZWKtu5aRt+cRp80q+LEOBDfhMv8tof85L9d2YjSRLAjIkktAs5t7uNKvYvt7hDdUYT+cIxmt49SuYR0mEI+EyIIs6i3OojTBogXM8Zm6PT6aDTaiFmLdTFApz9EkMRYmZtBLsXy4Qj3f/EreNlzr8etN5zQInPx6XO5GYLyJnwL08Ap9QSi3JRKJSsaOCtv7sqoNN4UMyjjPcvMUqkcOU2fRbNLBMixQgyfjBNdmKgCE+nBgCmBBSs+7DY0wlMeLFywENryNn6Q/dSCE2PBGZTl/cPkbwcuK/dy2ic8UnxVswiWM1pJTjxTS75cnjtFXWjaza8HGMUB7vraRXzykUtojyMsLSzIHOWZMycRmt2BhKdYyCIXptHuG4Hs4vo6arUqitk0Wkw9UhkcXV3FuUsXUS6W9GyDkUF9lUIeWQovEmxvbqK9vYHXvezHlAb6qN3TSBjV+lzVItIpbst4hQVvrb8zNcLKBc4TebIYwCg0Vvmh22FEzg3mWuvn1Ez5DYfG84Lk9zBCEqrvcEWZgUkJxyEOAaPTjBaVacrszOzEpwoyE0Pv20Fpj2jYZnJzzad4xhml3JeqKuWKrqvN4SaGRro2cMEB+NpYXW2iqTuDId7wsS9jvx9LkvuDPiq1qoRy4CovXKj1rR0szc1i3O+iOUqwNDuDVqeN4cgiUfrKdC6LIwvzePzSFeRLJbS6fd1PQYjYWPBnIZ1CpVLCg198CH/8E7fiyOI8AqIyDGTSjMTJwbXareJHuiKBNFZ/NfqIBZR5pod0bSrnuUKFAzXkH10qxI08GPFqBQgacFf5x1flubg0t55WafwaqxfKjDreprfn/qIGPlt5V9priaWkinmRrzeKqUZQgPirY9PxtcZTzUzMr0yHq7bYphuEZmx6q554K8HP5X3sdwZ45QfuR6ZaQyEXStsazRZ6wyFy2Tz6onCyVpvBxSvrmCmX0Gx1MQ4CLM3PYKZSxZW1dTEKIwpOmMZ8pYS52Vl8+RvfxDgxemkhz2cweI1anEoSXL26iVtWivilFzwb/V5b0S6FU8CI4x3T4um5HMTJNeS9+Borg0FlBirYGxzKTaS/9BCl3IjbWB9HaN1NM43DSdvuGWqWVrgKvqocVhe0QrXjuVKbHcxHu28Laj7HKhgGcPuol1rlAeYpXDUNw52NsQpAEEzbHHxN1Zlwbibvg3xZ3iej2lQqg3g8wJsfvIIr7QFm5CqMyNzrD3F5YxuVmRlk0inkHBDQ6w2w32gicDTIYj6H+WoNrU4HO62ekCla/nwmjZlyFReuXsWYwpckyOeyshpz87OosNAwGkgots8/ir/6pRcinfWFcMvHZSYJxijDscqTj2iF9jjgREVtVkLI7iMzXsGFwaNWvLCOAk9CY0DEoElK9tADdwoB8pVxJdf+w13JhSF1uVic8HMMN7UgxZOgLXn3PRvyCi6lmSJGinQdhUSRp8MphRqJqm85ncch+XO+hgGU6nWudqkbn9AzPYifwVo/wRs+9TVhxIdWVxBHrFEC7U4Xjf4Qo3EsCC+JGbil0Ov0MQxYtbAEPBOmUC0Wsbm7g9YwRrlURjoM5Bvru/tYPHQY5554QgKSZd0yiTE/V5MZTqeAze09PPzAQ3jHf/kxpHNWjPagB4VPbRdpK1B4rHlShHbcYg/AywciQLfTNrhTHCcLrAiX+vjDLBVTxhSCz97zPrHz6KcMjWBYbFIlg3mgQcYD79wQaU/KUH5fHVERmlor32Zpii8gKxEOjJ9LtsI0EDJA3PgyJF859oDjClES+Xq+XzRIl8BTan2OK2uRCvHKjz+ExcVVNNrGDCzQX0UxLq9vYWF5GTt7u1iYnbGfx8C3Hn8cZ697Ei5evoRquarNHA/72G/3kcnldf1iMYdsKo1Wu4fa7CwuXLiAQrEkqigXuVIs4OjSvPxuuVrCZ+79Al7/0u9DtZCVj/SCSe2xdMmCQGYMBBaoWbzOQOnLlDvLzfHQoQdvtKGOOOf5Taa4zhI+9MAdiS81WQRlHUoeKAiZebroyf/MXjdltvddbmTRq+WoFAwfWAlQd8AAQ3L+zmO+E21l2uIgQoHsrKw4Tfaht+W2ViP17AVLqyJ8vZHCp89vopDPoDsc4+KFiziysoz1vV2MEWJpYVH4bjweYrZSwn6jjd12D8cOr+LK1XUtarWQw+W1dWRLZRw5tIJHz1/E4sIsmvUmkEqjWqkoeqSw+K9sLoNaMYf5QgGlahGfe+Bh/PrzzuLmU0csonWpmYflCEswK1AuGpH/a5CcLJCDUvl7aj+BfE8CsxzaFa9dbOJxYV6bGy8za1poG2F4q5lJ5Xvkcna6eghGXpQoEqZUkHW5poB5F6gIbHAUCeG8jh7CjyAxi/niZEM8UcxVT6xBydj0MjeO92opkVUsmHr4RRKLIZVgmCrglR96EIuH5tlBJKG4cGlDZnJ7bw8LKwsoZDIC5tc2NrE8O4PzlzdRnqlhplRArpjHzs4uwlQaW40GlpcWMFcp4fLaFjLZtPJPwoFcp8XZOVxaW0OoLq4AxoCNcN3JoyhmsnjwK1/HD14zg397642uQ25sODXrp+qqs3qqcaNoBc0aKaLnOqZDhM698TU9UjdVyzRkjikMQf+N9XXh4TS5pmQxgvs+9b7Et/EZU7ww4eowb6Mj9ugKN4abSimhj/GsPlN15n2xTKyqCNRmtynULO+o1Unm2un4kAUHBhgsx2r7t7cBUvPKpZLgNWN2WgcU/8+Ug+DAG+57HM0khdliCXFCVkCMZqePc+eewNETx1CbrSIgeSydxpWtHfTaXYyzGcyWayhkTIAZbe+3ughzOZRLeVRypHvm8diFi4gccy6IYlRLFWzubiPNnhJe0/WgnDq6ilyYwqUrGyjXL+L/+qkfcHVLZwblPYyLTC3a3d11gmtRuIoLxZJSE+Wm5EOxKE/IznGffGYwiTUcdu7NcHD/vR9UNMsNolobxZ59mBaQeFIR3bGvUfKmbNMth6RZNqCdgO9gsuDeRPi0wTTeeDjOaeo93mf7wqwHMTxDQQ1IB7qo7GGM7v9IK8FHv7GOje0tXHPosCXZwxE29+po93tYWVpGrVy0HDRKsNdqo0XidiqFUjqrtKJUyGEYJ7i4vi1ucDYIUCpa8fr81U3k8tYuQZx1f2cXc4tLkwiS7Iowl8XJI4sopUOsbW3jiQcewJt+/Sdc849lAR6AP1jcNi010pbFRAa4eBcmiibxbw9CqByZSKF8diE2vG8e/uw9tyeiVTiWOTeV5sAHMFxoVg9k3/MFhIS+HH3f+iYst+y0OwLWVe2gTzPWo6SLTUKlYlGO3tM4hXY4NoJn7U0qIGLrkQE4cukJuaE522vxewjdJQpu/vST30CTLQvZInJZpiwRWu029hptLK2uotGo48jKilwEzRZTlFPXnsVes4FcKkSeZg1Ag11ZJHRxk6mVmQzq+3XkZ2awv9+Q0DJN6Xd7KFVraLdayiP7vQEyhRyuObyISjaD/WYTX/zsZ3H7K15sYMfIuEMe/RH7gemc49QS2vS4rOIKh+cpx3StjkR+eF/8TK6hR9mMvmP3LGH73L0f0GYS6poi/aZBMgyumOyxQp+6yE8KUjMaB6kmGW6ma/WWdkUmab4VUJGyq17Q1HjmACNWLowS61zWGnIdnEU/5ptw+VkGV1k7xacutnDPuTXUqmW5ho2rOyiV89jY2sHhw4fkj9bXN7C8vIRoPEKj2UY7SnBsaQE7rTYK6bQKzds7zEFnBfk9sbaGSj6nqLEzHGNxcRFraxvyVc3GPjIUSnZzZXMKqPabLSX9h5dnsVAqIZVL456P34N3/soPWVnLMRJlTRQbWKBjPaCxOuH43Nbid6DFn5guMXKCFy6CVZ7JYoMrWijfcF1n3ODg3nveJ9qIGtlcEOOr/J6/4hF/M1X0i7yBtNh4Qiccf4gsO26i+io9W87xT+kDzGsYDOcrLj7HVeWFyFPecqqUaxGgFZDZcaxxk+gIzSHw6k88jEq1hlwQoNnv4cqVTTC6pHCuriyh1WxhMByp26xWm0Gj00dvPMLR5XmkQnaB9xENIzR6HSzMzePw4gLOXbrMT0ar10euXEEpV8BoYJap0WkjFJCQwvzsLNY3t1T8pplbWZzBTD6LVCaN+z79efzdS251z2EL7pud2Nfi83FRUCZMe99O4TMCo9Co/1IuzjccGV7t6tETZqLU775P356I3iCc1PykbzejeVBV37GwKQls1ElnM9IkI2cZZ9Yzsn01wDe0agMdUWlSKXA0EvNDVtbypTOlLa7xl7/v9yzgGo6YhzGdDBEkKdz+rV2ca/ZRJKthOFDE2eoOwDTpxDVHxYuhWR2Mx9je3UeuUEJX9bCxUgmSwNi5vbPbVAV/eW4WhaxVjLb36tjcbyFfKiAbhAIadnZ2MIysQMznqJbL2NzZFT2zVimz6xfXrMwhFYS4977P450v+35HWeXcgekACwMRLN3jMw/HVmnyQaQxB609cQIUjIzIZiZ1iqyR0c7r+ZwzuP+zH7LURGw0z9IzHHD6ZWiOr4rww2k+va33qQw/3aor0+ER0jzROHxLoEW+AhH0EFNo0My6J23Y6yIWHjWEwfBYPujl9hB///kn9PtKqYR6s4nLVzYEtS0tLqBUyqFaLqmqwMBma3sffZqqbA7ztYpKXkRvcvkSHjl/AfPVCor5LIrsscllsd3sKFBSkZ1sCiToE15j9xiHS6QN5OCt0eKUSBYPElx7bFk+/d57P4e/fclz5JPZQk/3ZQtu9MhJXKGAx1KWXn9gRXYBI8bSU+whX016i60yr8Mo3gjhrp3D85O/8PmPaDMnvBQPYLNXRH0TBpT7CzH1oHkw6THUSMk8AWPX3xhhWtdkAEAfw7sxMNkEw7TSTEA72gUAACAASURBVCi/PLuAhWr6UsJefNl45ArgDkToRRH+7rOPI86VQLYBAyxq3i61L5/HsaNHcOnyJVx78oSChXq7i6vrW5hdWrCUih1m6RD1dlsBVGswwiw1MJNGnpR/ggLdIQYxKyJp5NNptLsdLCwuYWt7RwJN1Gev2UKxVFLuTJdRKOZxYnlG/N7P3vs5vOYnb0Y1n8PYbb6UwTkasR4c8TuOjcWRiN1gHFyXnBuCNJlhYOtG1+ezD8s2fAtIguCeu9+b+EBGC+t65qeNKyyu+tbtaZu73xAuEIMZ9VlQEsltdRVw3z5gJsR4pboRB/mZtE7rkso1M1lJr8cgPX1fZgkJPnO5hXvPbeDQoSUl9c1WB02mG80GbnnqzYoG165exfzcrIKbK5vb0qaVlSU0Wh1UKyUxBNa2dpEv5tWcS/tAE0vh2dprYn5hXmADNSKfzmCv08JcbRb79X3DQJHCSHXfMnqdruDGYimH5bkq+t0uHv3yQ3jDz9yKuVJJSb9aCEaszxqgbsUK6yILUlaYp5DwuQkVivRNRN4PpEhM2bh2W1tbLkrmdBPXdOvSmeCzn3m/gHamER77NBTI2FPsKmavvtcsZ5GdH+Um2bAEBU1i2RlpiwIgaNAFPhY+m0bz4STRzqmLu+MCK0Z8zCt9G6Evp/E1a+0h/uKOL+LM6dPo9nvY2Klje3tXlfobnnRWheIoIAV0gLW1daysLGNjdw9HVi3X3K63RK/sDfpododYmK2ikM1hfWcHM4Uimj0OjEgwO1PFbqPB0EsL3We0DTb2cgNGCo6CMC2EiZvJ6JvmeXG2imjYx6NfuBd/87IXCHhguwa1TQQ4VROYrpDJzpRlhGptVv6wXq9Lb0uVyoG805IKKhbLd8ak8DOIpuN9KMBMH4NP3/1ebSZRfPJmKSHGGnBNPa7Pwie9PkDiJvo6qEo6rh9EJtIRjdSO5/sMXeIrIODAVCzPSHAWSAQsaidrnXL4hl5gMErw2k98BZXFZYHcm3tt7DcaIGWSwnP9tacRR+wgS6tFcH1jW9FVpVbG0lwNGQ5H6pFIPMZOsymcNZtikTmnrmwyCgg0sJ2uUMipI6w3GGLfsQDoLmiOuQE7jbbuLZ8vGPtBPShpBNEYhw8t4Wt3vR+vf9kPKSrmevi+HAU3qtumJ3VaBkBqOBK31nJ4tWtQi7mOftKZawk04N6SNQMaLPgU++9f7nqXek1YMffFaV/T9LbZ55v82zPoPEvO56bSXFcZF3dIVESbJkJHbjmWm8XDsWsqyPrBSNbhJe2VYzEw3vsEsgM+dK6BvWGCvXrdFn6/KcYa0w/SPAie5ws5PccwirG+uS1WwXVnz6BSNE0nXW2z3kan30O1VFBBOecmZa3v1jGO6FKYGhH6y6Ld66Pe6U4qNTHfNzMjrabUk5HhqyG8ddY9a5USzt39Abz1N39KPSA+E/DBZOw6zZRqcayM4oMQo7GlHlZASAkLtgjDas3MDjzrkCQ01lIVx8jysV9mhOBepiYORVB06Ro5+b0nEk2BA4PtrAXAODrSrDH7EwcyJWqR921yjjXAmxVrbTCUCWWLva+IaCQK647yq6HBVMJeE4zVuRzg0+s9XNzYR75YxjcevwCkstjZ38P+/j6uv/46tMiYazSxtDiHVJjG1k4d+/UdnD1zHcbxGJV8Fvl8FjvtPjo98pwiVKrWmlDNZbDfH2BrZ09QHs0p+Tpk7JGFx2iTr2MBnJ8xv7SEnb06MmxnKOQwHljqRu0oMscFsPfle/Cml79wCoC7gM8HjbweKSlcs53dHRw+dBj9KMLszAxYMKdGZnMFWTCVGxlAOr9JK1IolieNUMrbfTT7+fs+mHDTGLQQgaedE7HW5X4WyZLawLCds3emA5PoCyhNI8dtNVDYSMDe59HMaICT62Dm9XJZMr2tomJMd4uWFRFzdh+5u2Zo8MFvbaMVZzFTLeHKzr7w0831bWGti4tLKFeKQp8uX17DyWuOioC2tr6Jm248qy6Mxy9dxKGlJX3Gld06jh45iq5gMdJIIyRRgq16A4tLi2IuFDnCLAyxvrON1dUjuHJ1Q89CtIiAAzVza2tH6cjA0SUpeDSzuXSAeNAHLn8Nv/p91wkoUFuko6cKnHGMDaZR0+cHkpAkcetYV04pzhBthHsdUhJaXqtSnbHCvhtkxZcowORmeqfK4KXgZud5DisX2XNaadt9sktw3fdBaPKWy4O0Bb75yPFpfeRLTFKkZjdLyPNtFblmyXAnWE/2QoL9OI2/+eTXcObMNVL/9mCMC2s7aDSb2N7aVqR66swZ1Bt1fbZY7oO+zM1crYYjK4syp2s7e+h3RyrLZbMh5ufnFKQ1Gg0RkpscJDEeY2l+Dt1ORwy8equLXsTrzCgwYZ5crlawU7d5QJ1mA8VyGf0R6Y4M8kYqPJQKGew/8TiOl/v4zR+42dI6B7LX9/cFDZqrYTea665WFYhLQkWIrbQm5Md4PvSJ/cEQ1UoVnS7pIUbm5jPIDWkWxRDLy8tQNOvNpbTDtY77iogH3Pk3/aWn/RkYb+aT9Hivzco93YQval9Jc4TMHlsngHFhzF+yD8RQJAYvUZBGd5Tgnsd28OCFqzh24hrUW8YtGiXAxtauhGF3y9KNa665ZjKyhvjl5sYGKuUybrzhLIa9njivO60Oup0+gnQGc3M18V0JxBMpYqkslc8jl8tgtloRQEAt3GowhyTx2nVuj0bYbrSRzReFk5LM1ev2MYwhLhBhwTSDrXIWV770OTznycfx87ee0Wv5jKxyEA4slctuNh5RIJv3MDM3LwBj0B+5EXRUGE4mSyuNIWZbrpAFkUGsxienke5vxiZMjWRqP37nO6WZqjOyVukwWgMEOGNupNTEEJspuODJukr4CQyQj+or5Z7aIZTIsExKGE2ubaqVhAhU25i1NOrjBF+4Usd9X30cZ649i86QvY1D7DW7uHDhojaWKUi33USj1UI2lcXM3CxKlbIbkDjA5vombrj+LJaXZtBodNDu9rC2saPXcVHoElT0HvRRKFcQiSYyQj6dlclKRmMsLC1hr9VQAMT+TGoF06xdfmYmK/SlVqxgr9lWGY4pw3Dcx2y1jN7+LgYXHsYzbroe/+Gm1ckMBJlWQ8XNPB6Y59frjZArFdWJpiBHLR8W8VNT2Z6QCjOa8Ml4gKaYxQjlrW5oZECMikpC0EDDIdyHcK6AmUlDbHwHtYXXvpV8OkJFqD2FQB1aRg+xTTO0gteZSLgzxQLp4wSNYYKL+0N87vwatvc7OHHqpJLsYZTg6996HE++8Uace/xx1VmZVnAs2/raOk6cvEZQ3aXzF3Dy7BlJ+O7uNm556tPQbjUxWyui3x/i4uU1jKIAC8uLaDaaWhj6Q3aczczPg7K3t7Nrsxjor3NZHDpyxEwYn4fROAnYuSx2m22ZFsYXtXJVcB/LhgJUUkApF2L3G1/EmUPzWJ4r4/+45ZhbQ2PnMcXwLsoLPe+buEmpVlXFhEwIQoYMEkVxccOYyUBQ4Ji1EiOtmno+w5TydVoY0Tfv/sT/sjzToTRpsd4MCPBBi889Lfix0SV8DzfYd0Lz5xowMRnpMmUMeIYAzUSzn+CRzQbu/foFXG32MVsr46Yn34jeaIj17X1s79aVbuw2mjh85Aj67bY+a3d3R34lky+gNjOjNGjj6lUsLy3Lr83MVrG8siTfyXti7fGJS1d0j9VSUcyI/WZduGq33UNWuWSMIaG7bs8i8WoZ3d4Is7NV7Nfb6I0GmJ+dwczSivLZdpfz8dKI2J09sPUhZsxKzWjrEpL9NTztlpuRG7fxwutWDI50gy74Gs/Wk1b5Dm8OZ5LAZ1CbqU2GOAeBNQZRown9Wc+MpTOexSiMXLMWHCn9rjvfmVinsw1bopk18MCPIfX4qQ1+8jwWT4zmwnk2uSd/eQzSg/PNKMD9F/dx/yPn0RgkmKnVsHpoRdTEQ4eWsdtsYm+/hW6vK8Rkf3MbxdlZm3unslsE9okSfz1x6rTRUmiKWN5qtSSt15w8rojVF7q52fvtFoa9PpbnZ9UyEI2H6LdbKJeKjtvUwkK5gqViGoj6WKYGkzqSyeDKfguPXtnFoVNn0eoPEAUJGs2uFny/3VNEThfEzUz16tj91pfw3O9+NgrJGNlgiBfdePwAGsY6rxvq4eg1xIWtLS/kODQpiE0Ns6ZbRuKamcT/EXLU3B8378HNqbVaJufvmosMPvGxf9SIUm9CmXRbsOOGALuUwYME/udSc/7O5Tga0uD4OSPXMbablHDHw49ju9lFtlzD4tISOr0u9psdwU8bG5s4cuQIrm5sSGqJf4zZkdXtYJTJqa+SsV4wHODK+lWE2SJqszOGSbIBdzDE2uUrihIXF+elwa1OU+ae6NPe5hbaOztIohHyqQjPu+Usbj4yh3I+jflSHsVyCUE8Qj7rmYbT2X2Ufs4+2GoN8Y3NNj722Db2esDx4ydxZXt3knKE/SZ2v/ll3PLMp2KuUkAw7iKXGuKFN550NJq+UVIdOY3fW6Jv2GxIgL9AZMmK0SPXKslJmRpkJSvoOLPslSHbIwxFjGN50Mhgbj7QXXf8Q+L9oar4zuSaGXVjvA6kEhbdmlpnWJpxZpdSyvCZEewwDnD7N3ew2egjW+Jk6QzW9/awvbmrmT/MnhjOl6ozGPR6AqcNhUph68oaFo8fQ6PBCn5OkWNjewvZSk3oDstdbA5mxLyxtoalxSWlGZUqGYMZNPdZY0yQyWex9fg5lKM+fvlFz8N3Pf1JKGbVPwim4jF7PFiVGA3ceBvF8jbn3bVYiMCmSSQ51Xs/88QePvBYD8ZyChD029g+9zU865lPRbFUQDLoIA1SWIDvPb4gBWEdVhxftRQYYY5oF82qrItr+eD+MqckX5eBHz/TdRtPgAubPz/tLLAhU0bTZBwgOI8SIMCAUdaBeQBGtDJmtuA1aqwLbmyzra6n6SFia4cYjBN8YmOEtb0Bzl+8iHyxhGbbBjkQfmPUy5IYA5LVo0fRaTUn6FEyGIFLSfYA+x7VgRaGohXSvPL7zbV1oTes1IyiCMsrK4pC63t7YrDbNWJkx3387PfehBd8xw0qzbHBNlaFnvNuCaiz49hmAHW7hrWGadskPiujVj6jEC9QSylwGey0x3j9g7vY29xGajzA0295Cu0Juu0G0nGEfCbCYi7A866/xvk2izp5LSqCH01OReG6sTA+IngxJo6bRTqX0XTNdCavoIfRldoTGeQ44l2vO1COb/P0p6NhBbQzbDf/prYtN6aT7XyWOvAhZF4dScsIuX7ENOE52nT70I9dGeKf77oP+UoVG+ubKJTL6pCygYjWP0FflyvklSBTQ6hJNK3tdheLRw4rR6R5bTXa2N/axaEzp1WxYEjfbXeMQUAGfDaPaqWIcr6IXZlTSztm4j5e/cv/BkuzHCnjTWeAXrejvDAVOLPk/LH1TlrHNglWisY1u8ANQxwxV+wqLXisncFf3fFVPPmG0zh2aAXt/S2M+j0k8QjBeIRaIcCRWh7POHHIaDhJpGf2AabYBZo2ZpOsGdwME7oYFihymrbFqg/IEWJRggElAqVFaQ13tsoONZzvZxTsp6sFd3z47QLaDeS2hhbfa+KnGvv0gukHN0JsPkd9kHGKE9nwRj/Gf/2ne7GySDb4BU3rKFeromgwZ1P373CIer2D1ROHMezbsPhRv4v6zh5yM7Mo5Gx+LP/sbW6gPUxw4swpm8VOs9TriS03TGJUa1V1VQfJCMGgqzTkRLqF//aSH3Wzcy140mwCTUIhQO64NcxLYnJsmYS7Obg6QcJmrXuQX2kAc77xEJ/biPHWex7FkdUl3PSU67G/cQlJt4GMgocxUvFAbQknagVcvzKvaxB3JiatYE7z5k2QJtUk1yTV7Y+wsLCgjnYWyMlG9J1hsWbU8ogQg/esW9CYGr6XRSQxggZealQcFsPapitSlQ9yczTCpdeb8GvtHBTTWtrv/SSPl7/h/VhZXcEoCRSgsNWc+SG5uGTIMSjJFSvI1UpIB6GIye36vgCBbHUGJRK6KK3EW8+dQ2XlMBZXl2XeeU/1rW2L+JBgaXlJDPZer4Vofwc3r1TwOy/9McR05a5AzmCDn8vN3NvdNvagnCJ313pecnlrxGEbnRXOrdrD/1gjzxBf62fxDw81sHPhcXzPD78A3f0dxM0dZKM+406kkjFyaVZbAtxyZAUnl2a0mZ0OSWWc30M2gmUJPkXh35msTaoejKxRSd3e4gllJFjiJ8tPAo1222YiuJN4VF1RekIeUGQ+U2i+M6MM6fmcuYxNc/Y8HV9Y9rir7/VQCqNWtZTyxpf/zUdxw41PxtY+Gds5tTaQGKVCda+HRruL1cOH0Wm3NPqFi7t96QJmjxzDoMPBDjmEQYKrjz2GleuepIXlRlfKJfT266pkzC4sIHYz2+PBAO2tK3jSQhp/9J//g9UKD/CVNEWM4MeIfSbcyLEAdoEkjkNDYhT9kw9UrBQ0pWmMwwxe+aUhNi5cRHtnC9/9g89Hf38bQb+JYNBBPpUgmx4jHRi8d8uRORyb42am0B/YEGEKFeMF/s2R5+Q2sYTG2my90cBwYG3tBO8prKHzmcsrqzKv3FjWPEmFIWnMz42Q2XZ8LIEGxuM0Mq3Sg/EYxTzDZTvgxQhYzNMYGpvT5Rclz7dhUzsb3RF+5R1349DqYXQGhn3yWvSlnEPXaTYR5EqYq5YV4DB/Gjq+6OzSEqL+EM1WUxSOyxcv49qbb9b9kBlXKuawu72L6syczPag3bVgorWNamqEN/32S4T6qJXO1S7ldMjSI8Afk8NKLDFCdtwSmJ8JSfBmbm2+UX+7Eag2/TIlYXzX+QRfuNrA4PIVlFZXcGh1AbloAHSbSI3bKGVTSIeslkIco++74RqU1bLD4VE9pRNEiSiUvouaVk0mngM+VOu1uEOVEo2J4fccB0sucV7+m3VMC9QoeEbmYvzA9IaBWvDB29886ZzWpoppQF4KAXPepG+QtSiPFH9WGdj/oaBHQILBXilEeM0nH8MXvvEEyvNz2NraFUQmRhslP4EoGWS78UHIDm+3W6gtLIGIpIjK9To6zTYKMzOoVMqKQhNSNdi8ky8i7c76oL9jG8HSbAnfceO1WJyZxdVmA9WZBeQ17tTY9PuNOmZrMxq0a3PXjRFI87nZaIqcRd+t6BwR0sOOhlsVghFWSkI98dqv9lHf38H5Bx/Cd/7A96PTqqMUdxGOegjjnoSPTBsKA0lhP3rzGRQyNq89cicS+UDIt/l5nxmm7IwVDshQwKlJYVnuolgTvM+s6+thaqKDguhDWSUa+gnb1kIffPxj/2glMDeMiJspAMGB4Yr+DpzlYXnN2LHITIupueoYSyW4sDPAb//dh3HtTTfh6vqmURqzFokRwsqFrqNrPEar1QSyRdUGg2SsUlNjcxODMVBZYACRQpgk6O7tYJikcPjEURw7sqromMjP0UOrKBdY6TD/xla+kjtSKRuSomit+Ht7DQVoZOAxH2uSJiKcOY3ecIzlmao18UQJ4lSEZr0llkGWfj4CHt5uYtjYx/bGNk6ePoHUsId0v4kM/WU8QLHAyDSSe+BmPu/UiqozGtXmxusoOm+33RQS62mli2L6RW09duKUoW4KLEOk2JikwwYSaS/XsdXpmgbCymCpwAjhfiLJJACiBIgm4toSyI2hCTVfadxOaqYVT/1ESuv7sNk3dNpEKlJ42d9+DCfOnMXFq+uTScaDcYxypYQwiGVWRr0u9vbrKM8t6IAy8nHiQQ8bFy6gtnJUgRPpIBkJzxC3PPuZImWR30rtbHd6uqe5ckkIjuW6Mc5fvqKokP0iLADI5FIwkwTt3gCLtZK+Zw5NNvqj55/A3OwcarUKwJlAmk6WE4BNljyFKFOdxcXHHkNnGKNSLqAwaiEctBFGA6STsZqMIgxRYA6dCvGip50x2IGpVI+Nv0BPM2XZkOWDKjes2eegTP/CnCZLKQALLO+Xn8znRGDTNM5MFvlCUVWgbCY/gQx5KEJw50dvU0sfN1HTMNwIbuWCPNtKxGPbTBaT1eXFIe9yyvw+pYjWuLRE8yO8+6F1fP6RS+ix4kAuTbeNuflFzZHjTIEgirC9voHS7JyA7yHLPEiwf+USkkweK0ePYGlhDqdOn0SxmFdl/8jhZczxfA83XKQ7HuPylXUcP3IIIZNu5x81rInzcti7qNQgAsP+i1evYrvVxeljR5BOrKDLiSGE0vbIxMvmUM4V1ALf6ds5JBSycqmC5ePH8PCXHkJ9AJSyAQrDPYTjPsFhZANOJskhDsbyl6k4wr9/9k02fZJMwV5XG9hxBQNuLD9bcUmxqEiX7RM0qYVCCaEbVsEZDRkGgyzwMxKv7yvf5F7QvIrwhlA4OjeW+ad8php2XJOtgAPHHKfxIowlkzThsUwrLH6urCcD+cagr2718Yd//2GsnjmDQW8EkqKJp7LFXDSTZkM9j0z6Meii12qab+538bRbn4MnXXcKhXxagsUGoksb26hWy6gQ//XHLaWAZrsnNl2RqYWbBc/7J3UykyuqjLS33xByxXYCjvgk2+6mM9fIEvC+yVTf2NlGd5RCj8k7cVDXds8N6TabuOUZz8AnPvkpDMIilqpZBK0NhExrRkPk0oxgMwjSJIGnkIki/PDN16vYTkvBtncPyAgFcnRTbqisoa8qsruGayAEilqaVZ8Mgye+hopGQbWMya7pp5FRncXO+9hH3pEIDBB1w+a9MWlW6uF8qbH0/KcaUsT5cBz+ZFQSBkJG8OI1+lGIn/uLf8Lx665HvdXTnDrVMIl7xjG2r1yWec0GCY4dXsTJE8dxaHkJfW52No8CzWZgKQ+plt3+EFEYYpYDI4RtWPWg2WyjMxphYa4mfytCNQcgDga4slNHPwpwfG5WRWSNHB30sdNoYGlxHiWW7zJpXNnYxjAK5M9khXicFflBvFoKYh+cPH0SH7z9w5g5fgLlZIi4vSUTS2plIWMzGcJ0oqArH8R40bOfoXZ7G13qJ0a7IfvW46FcXVmCqyXT76tznfEFZysxT9eQY6ukkEIi0F0Yr3GO6FNJm+F7mccHH3n/WzWjfXpCrU3DsgYebpI5aN/0Q4kwTJBY4pQ+yYWctHWHKbzhrq/hW+sNZGuzAseptamoj72rVwQcnzx5DV7wfc9FqZhRGwBjTLHh4gDlfEaBhDBNmOM/d+kKrj95EhCTz7invL+9DnPQiiJvBlTs9CKYzxk/6WIV5RyxYOgz2PqXT4W4srODbLmM7Z0ddLs2XobBSj4MUCgV0GI1QnNuhyDf7tobzuLdb38Xjj35KShwE/t1hKM+UglNNYdMMXm3sejzhQx+6BlPE+DPtaJ5pYJMD6C1w+n8YUCe8KXp6BpgzAI1/TmzBOc33YxfpiQat6qZhgnqjeZkr+TyPvDeN2ncmp22ZxNGLEMyDdCgJXcEk2ez+yledtaVG4Srg07txDimLo9t9/H777gTNz79GTh/4bLMdTkd4TnPfqomeRH5KPBUIR1CYNO1yBQnqMCuqlRkB7uYhQ9wfm0Dh1dWUaL5JZFY7XAJLm3uok64LM3INyWgWg9ab2B7dw/pShVH52cw7PPUwDwGvT7Wt7dRJA2D7Xqc6twfGOTGYVHxSMMQU5kcKs58Hz60jNve+o848/SnIzPoIunXkUv6yCJCPstYggvGMRgBjs3P4TtOHbNTGnRU8hANNva6Q9+I1nDhGVVz/by55TPR0rFdgZUU5ujEZ2k96A+p0DNzcwaJBilsbW6JRrLASZcxJ1s3/WZa5GVjSd2AisnYl2kkS2206rklr7lcwZVr0kI2otj4QmoFHMX4lTffjZXjJ5HOBbj5yU/G8lxRvooOP5MtyH/QHNFscN4OJ3pwpIuaeEIb2ivAO47dUKYaSlmjnDBA4dwCMtZaI+sZzXJAqJu3w2iXk6ORr2C+RjCe9H5GwW0MugOMhl3EubKxyNUkxD4XVoXos0IUS2V1U7Mb+/DCAt765ttww63PRapTRzBuAr0magXGGrws1SqSSb5+9RCefHxV5TxqZL2+Z01WBCU4FWRg5GVuKIVVwAtHdnd5HhknkqVV82U3HBuTaGoJhghy5bEegwGabeMzLa2s6v0s6Av0+diH3+EGIVqjQJ+QmvidFjmxZETtIwnYjt+1AX3CMh2MxA9SusLjlSIoQmU09tmtGA2wTc1wVeo7R1GPhgPkKmWoDhNzzDZl2uiSaxtbmF9aQNmV1zR+TcdWjdHsDzXAgVzWUWImHsMh1teuora6ogkhTNKpsaT9j3luyHiMbhKCeSf7OI1pHyj/a/OoxUIFRxc5jYRz3rvuzEzirFk8fuECDh85imuOHsJb3vR2nL7lFuQGbaRGHYQjcmwJe3qELBHwcevpYzg8N28gioB14xFzfSxC5nnZNLW9yZQtz4RUgMShkUNrpmVUTp4u806W/Bh68jV+0gkLADak0tYo+ND7GM3aOBYd8eQaZz1Bl0MZfLuAzayzRhZNcXbf+0Yj6lKf1flgBhf7KWSCGJ0oJfCcksMgRNKXABeuruPY4UPaTEoeLTynTxPWypZyyLgRb5q8MR6j0e3hrs88gCMnT2pciwSPZ1YSlRpHOHRoFetbuwZ7aU6fkbr7zTqG6RyqczOoim0YYTAeqC2BjUbNLseS5mWmeb9KylMWxZOLxCbe53zHLXjz37wN1z3rmQg7DST9JtLjLgrczLSzKnRViPHca0/gGIf960QDtg/YSUQeMiURjYX5VtvquHRL1Err4bRTHVjWotvT2Bg3GpYRK7m7ml3rOshIxbSTjKxEps3kRXOk+amH0HBKXtxHtf6YBp9v2t+WpPN1VKvxYIxGYQFf3o2pmsgGsRakQ4XViGVSIOgLRqBbC8Oi6Pyc4xMSydDotgCXr6whV6mhWspbt5S4PB0M+yP1Yy6tHlLIXm/uuyG91mOToQAAIABJREFUFnFur11FML+ImWJBM/TEZSrkBSjkeD+FKrb3G+jz+ENlbNZFTdRmtz8UN7VGkpdGgltXG6/B2uPS/Dxuu+2f8Izv+W6E3TrCfgvBqK1Bi5kUC/dWveCsn2cenkXWsp7J8EPNt3cFb/puOyXetXQQGi2XUS5XLd1wvGIJv4YoEkTIYnd3D9l8TiU/wqIUDvaNWnCVFvARfPj2t6g9oejQCSb2NtvAaCOeK2v+0gB3fwK7BT+UzBQeSx/CY7sDJBoEkqCYDpEnuEx/xmnOuZzY5py3c/6xR1GozeMEE/iAeLA1EFlOGwqWIzmZAUynS2SKJnOAnc0tVOYXRWgOYwLPxDKBuD8CohFqC4sKatgZzZYJHRsVjTQutNHuIShXUSaOqlTLfCVZ8CJt5wqYrVUxHvB8LTuBiALIfpZrz5zGW95yG45edxaz6Rhhr4l0zNMLQgdP2vWITb/wqU+S37W2xb6CQWHajsrJKJlBz2Bo49X45Rn9GkXHdKdQsNSF7kw8Wlong/rEjOjZYW5MYwjmjIYRypUygjs++DZtJhfU+0BuoBVpzfx6ygOBb2sfcOdOKhhK8Hh2FQ9eaWg+Oaclc9MXq0VEpH6kChogoUlaqqJE4uJcXNtAdXYO5RBCYeiTGWkSYiNSs9YaIiCE5XJTsdN0Wm6M3PwSijr8LBDYwQXrtzto7e0hv3pY5o5IzJQ9ESHNgCkIMVupaJCEigmu6jCORxp90xgHKOVLKMl8UkuAx89dxPc85+l44xvfimufdgtyURelqIdU1EM2lQjcEAacIlCf4AdvOCUs2tI5junuTDqiTRmm53lpzg9dgSavKJLSerOnRJ0DOvyV8xzY/lDS/bCeyaYmXrsf2Rxb1o3JwA/u/NDbtZluPp8LeqxfxM9FpwAZMG2ggL4jKJwKsV1axt3n62j1SDtMieZPTinNTy2fx0Z3gJT6P0eIR9bmvVAtostpD2FG5phWeDCOZAY3VLwu28LSQpDk5M7K1PyuUQ+52XnN3+EYFpo20Qwp4d0eYob3DPM1yozReSAzS4SIJfpRSDyzb5O1JqciGbzHoRTDJMTyvE3u6rS7OPfYRaVTH/3AB3H0hqcgF/VQGLWBURflQhqZkO2KgiuwWCng+Tec/rYZd72++UNbMvPzPp3jv7n2xuOxiFcsf3+iLoNClhAFKNA5pKxtImXxCjdTA4YdRyt4922vTUR2dsfR6zgMN6LUIlp3AjnhPjuKYDLxgqHyY7lrcN+5TWlWZzCQ8261Ozh5eAmrtSI2Gm2102XTbJNnYJHIp9A8cy5szWG8e/U2Rgp6LJBIirOC/8hsENuBkTRTgPEY+WIFkZL8xLXe2+Ap+ji+p7a8IkCf+LKnoHDBWTxmHtsPs5gv8gT19CQlEP0iCLDf4PyCBWkbc88LTzyB77r1Gfjo7e/D6tkbkRv3kIo70k7644ACpYN0A3znmeNYrVjBXSRyB/4T5aGF4SYa8uPPYDnY7mGkcZLeRH52Z5/RtLKVgga51bQTlTjtxTR8Ot1LJbDb/+mNmpLkD1sRdcRFX8pt3NARSr5KYa5dnZvKDemu3oQHzl3GY/s9NJQrRSjzNKB0oGAE2YwOxabU5cn3zKawVGLJKMQjW02B3oSpbGAwMOYpRq0mxgU2+bB670jYGtrLxNymlhRr85gp5hQ9a4IY74e57qCDOMyhx0ZaDgqWQPIR7XiqbJRgdxSjxgGIjpHoz+wkhMh+y6tbe5iZq2HY5fy9c3jRjzwfH/inf8bMydOoBGPEgybKcR/FvPgpuvZsLsStx1cwjmxgRTZbmAw4FqLmmou9dnpLR0GlAvkRBBoK7IrScnE6q4z5KQmeaeXxPedv6fKsBJmS+Q3e9bY/T8jR4Q3xA8YDknZTk7MwlQP5kw1cFGsNnkzUgXpmBo3SUeSKJXzl0ha22x0MekPEqQD5HCc0ZtHsUqLI9+E88yyKmQS1UglP7DSUU/WFq7IHMlShN+53MCpUUG92UEzzlII5tYcrwut3FWDkSlW0OsR9+whda72ETzSRMQaZHPJMP5jyZBjCc65AREhGYEU3JrCdiHRNqgaH7jMqtVYIC7zylSIeuf9LeOkvvBgf/efbUT1+GoWohaDfQik08rQ4Q6kYzzoyi5WZinJoCn6oxiMm9EYbMboHuTzWsk6fKAqOG9tNq+Db9wxxY55qgROBEGkeAz/ORBK1x47NsrlB7qzsOz/wlkTEWhi2SNuvHNP7Sfp2d+qeHRnFi9h5J9TmYZLF354bYblaxlK1gLnFefT7I2w327i8tYswW8D6Lsd/hho4WM0XEaditJttzbzjx9lZKoFaEWje5ktp5KrzMnnLs2UUwpRON9AYbxEqEmQKRY3eZjTMGqJACc1DCJFKIqRzRQELaWoO2wXHnEtn7yWJrN7uI18pYUwcNhVrM1UtSQVoNJq4sraJ+eUFfPPBh/GSn/+PuPeuT6By6AjC/h6CYRfl9Bh5+o0gwKFaAS+4/rAB9TwOy+gAzs9ZtDqFSP1hOabB/Dzr3XGUUHWP0xwaKMINZU2Tm6sGXfpKHj6gmGbadSDY88Pv+WvNzqM54034yJUmx4ZQeKKzoQ+e/a7FJ0kLKbzlMccxTWeEIFUKGRw9vIqV+Vm9p+k2t6GJkozSWImDyj3Npm2QMek5VSOLudkZzQa4vLmLUjZEhcVfnQFNrUyDhSIm/ft9S2vSKZtNQHNFMzUcdZHhSUFxiHEyFriuh9XicHDVWAD4/NwitpoNpFmHpS/mIEXWHltd0WF4v+1eF6leA3OVMspLh5B095AZd1DOErcmcyKF7z0zj2qa2jgdmGzHx9gXr+mZ5/7fDHjswDrmnDaDViUz9mGqVY/jSdMikVPLbdq1+VpRMCksrhtdGDCDwPe/+7U2otR13Poh+Qw2zCwYYOxLYD68ptlkzwtGY/zD9pwNaiASUchjd68BG4lLAlgGy+Uyjp84ovk7LLTuk6XX7Kn0tL7XkJTRBLOhh6D0Xr2J5dkq6p2B6pX5jPl0a9JNBMKz7pMu1KRtDHao3b7hN0lGyLAdLsO+yo6gQU4bUcM9WQcaIzfAqD/W4TNMYzRJWXMDYgxGfb2u0+qw4Ilo7wIqCwuoHj6FoL+viLac5aSuFIa7e3jxrSdE86ArMLKbGwbsGA06AYKnLrjNsC32g4SNu2sbTnNqfCoNEhYVx47UEoFrctqEEb8mh80xaCS78rY3/oGRoF2OIzOuQRVm03X6gcs3qf6eeik154cFAT6PY/jGlW0VT9XS505dJDubqQiJW0xyWbXnAPnDC1WcPnFMdp+MMw5I6o/GuLpLVIcIDFRNqfeHKLkpYcT/SWVhpKiRLewBSaWx0e7IzLI1gLtF3i83jtrLCJb0T7mMeIRiPi86CNMQNumwBqsWAM7fYY/HaIh2q62Oaz4fZyfke5uoZBJ0+hGKR08hF/WRizqoELcfj3D73/09/ux3f06z3/1se5vk6doG3KJ7Nt0Eh3VHavWHlgEouBTGPTXLLHUxl9D5nlorDgHhJtroGaFOkwktNLPvfo0b6+3MgaMbMkUwtH96xpbZaZosIwmz9MPzQDYwjy9sB3iCgwEFR1lXFVngjL7YWsCjeKlxG5vbaoOTVCUBBt02jh86jGtPnxAmyiCgN0ywu7eH3U5/OsItHqJWrqi2KbgxHaBWKOBqvSerUiqY32TQw2uwmsEN51le7DqjdpNtwPtmPycXjmkCUZdjR49i1BvogBpyWjksmPTO7vZlnF4syrdxgFRh5RqUsjGK4x5quQAP3H0PHv3KV/Gbv/jj+K5n3az7Jx7MaxODVSSqQRI8M8w4P0Yqnx7eRhqqby9QK19q2tSszbVQSGZa40o1A8iOxuAH6VmJ39Jy3X7bn7mWPotmdXSv+5JfdFVVYxtMTzI3k2BdSTTD38xdi8e36uiNh7i63TQ+kYjjgXU+sQdURQ52UwcKQhiVjeKxonsdBDoa6vSe68+cwKpOpg3QoA9kDbA/wtZeXQdFy8fQp4jSnFJ+u8TR3VwYBVWsjNh0MA6+ILzAcliKI9JIW3THboxGLD2RkW5DkOv7DcSZEI3dOrr1bRwqDDFXKcrkrW/uo5UUcGi5hmpqgMHeJj7yzv8lk/jsp12HP/itn5uMG7cI0gBaTVUB0GxwNoPvOLfZPra5brKLmw/kqZRcvZgmRRNZeFKFrbUCIWmnNTlZ2mVBanDHe/5Kmsnyj3ibOmQ0P2GGHzxkhq/zBGhr9zMBsdMSsthIz+HyII/Pf/OKIRuUFgZX7mhGP7CyUiiq2sGb8Qd8KqR3kk22AXPPve1NLFTKOH7kKCqzZZW2xolxZTr9vnpZWH3fbdQNUiMTT/PfA1TZSUbfyMGBIcN5I1xpBhYDN7XB8dC2looELAw3+l1c+OajGGys4ezpJY0yzbE6lErh8tUdbLTGuO7MUczGHXzgrW9V7sdFYP31LX/+m4r0xYd1BwOYMFtK5U9w943Cvp3dayphO8F33DjtoZ9CYt8b19eoPZq354IfbaY/puuO97w2saKokSzVsqfJk1MIT4rtbso6o3gxM7+W/DrzS2lKBfj67hifvdDS0AlBau64KEqUehRzNrSiRAKyY9KxLMT9YH8L+zuvbGyJDsKbZkrC6FxzetKh2uPnZqroDvq6tgYvCngfimHHC63vbJlPV///WOaK6QfHi9M7kW7JA9roJ3vNDi5dvID23h5mczEWqgWU8hnkWKwO7fztb17YxCCVwXWHZ/EDp0r4r7/7lzoPmwEYpfBPXvHzOHvm8GTipwZxiLFoU1YIS6qm6c4G1QECUgQP1dn4UzvwlKpmAZv9yzSQDRWaK6gUkmVgO8nIrECC4M73vs6ZWUtCfY+FbajlSpIsx9DTpAy3sf53suqub9O21trQLjaG+NT5NrYHJPJa8yg3gAk8N3GuxrKPsdtrHADIqDabEZ+2OyAHJo1CMYf9VkcbxY1ot8iXTSMJE1VGMkGAmZlZnZCgIyNE42e1xOj74gpp+DAbiOwYRCbynKW+sbGFHhuW6ELiEeZmC5jJ54yCogg5UtpDnu83zm+gPD+Pn33mEk4tlPHy33kNHn/iqpuiBfy7H74VP/fiH3UkLn/Yug35l+9zo+U09VNlNh+j2JFQFAjr4JI50yraHqSEAOlIZTcdW8ESZ9W78QVC47iZd73vr90MEFeTm2ibLcZB/+kj3ukmWjfV5DQEh9JYd6Bps3o9ogBfWGvj/gtthIWiQlX6r5laFXO1kvFIeRgpJ12y5U20INN6EpJJDWn3ByjnCxpSqFCdmqhDwI1YzEUj76dGNIvzZFtNtRnQ/Le7Xck358Uy0ElIVWE1f0SYESjN1DBPn0v0a9xHKh4KeCAdhAUoYrhr67t41nXLeP71S0phPvIv9+ONb32fJk1zF2YqefzD6/9A++BP3dN9uUPVlVf6g16Vvrg0xp2aoKDGIQuWnrAxwk0w0/e2TQbwGKtP2jlliiG4+0NvSqSRhIcOaJxjaFpG5N/gAhpz5E4GDgRL0xZti8EMUeKrlQXipb/6SgzTRRx9yjOwdO1ZFCozWF2a01Ss3pB1ur5tktKiNLr9LmYrNcFZOuqQeGs2jQoHTHimQYblLOvX4MweDhvOsR7Y64l9x1Ie/SKjyZBMvWxO6ZLmE3HNkgglNbG2UCbHddRDENlmas5PCji7kMPyTA7HqkxjrA396uYufuu/vQFt+mS5oQB//cqXY36+ZsLlSop8HgMMDBTwY7uNtG2D5gSjOt/ntkxrZgefp61lwfVx2rXdgeYTa+lOhbrnI2+RmZV624DMiWk1Sfh2JMP+bdxPr6n/+nUenvObbn4jwc/+n7+HrW0jOFGinvzM78BPvvSlaGcqakujRJJqOIgiHSbDfsS5alXmlcQmTfdgi0SOvCKb8mhjwKFAqtXuKlLlzADyZ7Z299xAqpQgMObErITYUGPybGIEbIMoFdQaD27kiFURAvo8djLAjUtF3HKMZSeS1izy5Bc35bf/6A06ucgOf03hP/30j+B5z71Jm8cxqfyG/pqtG/yylMSPW3MH0MRGmNMRGHKVNmJG/SaKXxjV8udsD2GswVKDrd9kbxJnkj92+xsmeaZSDwdDec3zZ5z4qMwis283v94+ENdVxd0NUTggB7rB//jLv4Pd3bqiNcrkU59yLV79R7+NKOHh3DE2oxx2hxzWm8bFzT2sb29hrlrThuZy5vvYRENUguZX0XVEpltf0CAjYMJy/Fw15JDZNnAz0slWYFcyTanOZWFeOhCjj2ebcDOJuabYdpCMkE0C3HSkgmedmkUYM4BKaaycITUGCLz/znvxjvd8fNIFfeLwIl71ey8zDSQCxQN4xjaAyZ/yzs3x8J6EwvW3cvi/Nkga6AdRmIHj7zxUKNflyNPs0xS6xFSFsc0nPvgmLa0tPPNM/2H2AgP2fY4zPRHOm1+/6dJS1URpctJyzqmUXcMm/wMveukrUK/vq8rBrx94/q14xa+9bJKTehOzPwS+vjnAheYIVxukO2Zx/MiqiwaNdqGSmgbdG0+nP4zVbDTlLdlJSAzjWamnprAAzu+FqAhxiZChFqr9fwSwGSgmUz3GU1aK+M5TNQRkHMYeKjRclKkYN/PS2iZ+79VvU6Gc9C2u3d/82a+rfsv3GNZtY9M0w8cBBvacNnaAwY2qHy6qZX5pfGQbTadY1s2MmAZN3n8SC3ZwG1/56Tv/fuL+pibUwmFBRqpo2IbKVDjTa5GvEbsMQPDa6sAEiZTLgUjhSId44b//VTS7baTdZv7iS38KL/7JH5amaZ7QAYfO7wXED8Z4bGeIJ1pjJJmSNoQAdyrtBv+r4Yn+zWa700dxo+iDmJdZxzEPEo/UlEMMlhGlxofzFjlum/hu1AeGXYRxhBuXC/iuUzW1SNjIM2sk8vVDO/Iqkkb8j9e8E+cvrUsT+fUnv/uLmt0Xj93J89RiRa/GKuBT6iADri2jr8CGB+skF66xMard+Dorg1kgRGviOM2uRmvuyx0HzfTsnjv+3gIgfdnf1m/pAiL3G6u9TTdTP/ZHDPvCtdtUv8EePNYYthTwIz/+n9AlCcst+Ct+4xfwfc97tsukfOu5N/QWzjOQUJiQEJscYneUxqPbHVxujZGp1NRYG41TqklysZj3+bPDyOJjLkkCFI/EoJnRUU4GiAlgZ6cY05Jg0ASiAZ5zrIwbl63bzBgDju/qTp43MD+S4PDWPn7vl/CeD9yjMhUX9vu/66n4iX/zPKFPrGTIPDqc1npPbI0D1+2sGZ86XcnyR96ZVw5uJIMfDUXUmV82r5Y3x799hUtrRJd738ffoaqJ/zoI4el792Fmik1bDa36/0J9Xjt96sIPo0mkX+Mhay9+yW8YEVhnqKTwptf9d5w4ekT9JJY7kU3gYUe26VFpLXiQrfD5rsvbSBBrjYBz9QSPb7fRzRTFih8MukiHee6/NJMjs5OU8VAJwlMryKTXERZ0BcMuqkEX//ZJc8iTyBVZPkrmnspSyvECwYrEWikw/iirRrOD//4/36lmJW5WqZDGq3/vl6W1lv+5qN6dykvwXGdtO6DFb6ZtKPkn5jNlhe0/2jxfHlPeeeDUYIEJDtgPPn3n27ST01EwTnIcgiGwwAHESsJd65/xNd20qG872sgY8ErUuZHyGwnWNnfwn3/1DybBAq/zvne9XgVrmwbtvlyIbkE7fZlhm17LuUCT7/0Mae46fVOSxn951Vuwcup6rJ69HnG+ogCDo7J7TE3SWU38YgMsTzlgdDgTt/Hdp6s4UrQRAPSpHmLjsvnxLbwXDSR0f2iqycCnRr7lnR/DV751wTQlAF73x78mEpmzc5P1c/7KugUcHYbnmfiNVK1VQst5s4p8nKX0JxS5kxP/1RpM4pb7Pn6ba0+Y4ogHc0yLPKfpykHtm+7A9LspxHfgtwHwwINfx+/+0V+av0p48kCID77nLSIhs4ff2sINqPCzFQz8DewYJtfvaO185vQlXDrVx6gi/PrDV70eDzx8Dr/w0z+GN932YQS5Ag6fOYvZ1UMolUt4ytljYtiv1kIcKViw50nRVIhv9//2GX4DvRBN66ZG6fjCQ9/Em//xDrVGkGnwf//az+L4oQX5WL+Wlr7QyrpTIUI7UIApj03iMiDA4Dz+00AD6aejl+iQO1fwUFQseOXA3tx71zsm0ey3Raaug3pCH/n/yT/9Bf81uOCvR8Txwx/5FP76ze+ebObMTAn//M43CoGZ1HPcYGHV/Nyo08k9Tca8jCaAhQIzl8OSW0O/cs/nvow/fd3b8aPPfxY+fPf96HXt9SmSrYM0/vC3fxY3XH/GmnYCW1CNkDHa/bdtJktk3Dg/hnXSL+JMmwKjWN3z+K3ff53yXDYW33TdCbzsZ2zgvg9SeA/qAnCaZ+aUrsrugdZYiuJOJuJm6v3OaMl1MftlwOaQNSG5HqfldT//L+9SGGldXGzpLjpJsCW2gNROyJkgv97HuuSf2+E10tvwyYe4G3rHP34I73zPB7Q45LAuL8/jtjf/uZ0RpmaeKZ/Fm1X7fCerHn9ky7uSbyeV7l68BeHM9V/+tT/Gs55xGp+47ytotziElxdik02AP/n9X8NTzp6wBhyNIOeiuXNCnDFhdOyLywyYTFhtACQ/zqJSTjOx1INTpP72bf+Mz3/5W4iSSKzA1/zJr1tfjQgyFnVa8GIuKEzbKU7exRAJtlqxL2t5IoBppwmDnYpEV2Bqe/AUYCC4/+53GwLEX2lOm8vBXKhNn0XO58EjpExKLPrUg7r3e0b85IacNlOC/udr34o7PvEZF+TEuObEUbz1jf+vNpMzYXVWpPuy6rlLhK2leOInCb+ZwFhOKzmjTjkJpo9T42kS4xd+/Y+xtr5jqEtC9ncKv/jTP46f/nc/ZOUmHVDOL3d6w4F/8zOsaDyNGUwz7SRez5rzm37uwlW86jW3CWPm9f7uL19ha0O43h0vwusRJ+YrypUZ1XmNYkq4ZRo3iC7iDl33KeFBxM23Vk63wO3DFz/9XttjhbuUIwf42r5rsQ6aT6WPExTDL7hbEndssfdzvjTD9/ze/3gN7n/gy05KgafffAP+9FX/j6FBB6Jp+6cttBZcgDdb8ByHVL7RBjbyi4sr2os7PE5QGjUijvFnf/V2fPIzD2LEESww5t8zb3kKXv37LzeQ5MBn69vYTaB0AYbm1Lm0QlO2BkMNMeb1PePOBjDZ1yv/4h+wvbev6/7Sz/wYnvKkUxPYk4RxWh+iNtZ7YtFroGmhhv6wwmNdVtMgdIoY+d7Y/93WlQDtWVXn+/17NlKKA4iKttWx01oda0dbdOwUQadVq9OCuwOWJWHVoGGHksiAyARlEVGQRJE1BgIGULG1VoIBQwjgvhSLKFaKCyQkIeT/O8927/3++juYf/m+93vfe889y3Oecw5YlA5NYFo6B3Gw8eureTKBYFBVGl7yIa7gez023TcxxvhoPBxUllSSbkZSokVfesZHyqbN39W7B6W846A3l8MPeZt+tKOTS0uNynNUd2epYuGRAq6JRopLIe/QoQsKfoGFPr19W1n31Q1l1efXMjTZuQuo0aDsNneq3HLdxUrSeTMblUN9GSJICkGEGrHTGLpbolETAQOTsEiB1D2uvf0/y9e/+W2aq+c/7w/LksXvFRvimWfY511cK6tdNqTAf6aJONQT8audUq2BJC8hH/BoYrSuNkjueXDnV67iAWQPg2SvyQYDIK2pCop7QsNQk6f6hTZspGdoIi3VtFF9As2uglpyytnl/ge+n70s5yxbWv7mlS9vDgf3vLsuxQuBu05BHCLjjirsZVwqhGpmAMzWs0Bgl6d3lQe++8Ny8vKLyrbtsHGCFFG3cvvqTzBvWrP89o6TEMBT8ESyk5gGsHF+yPbtbMyB6/C9VWKFBaCM/4zln+Lmg8G+4sPHcfOwjur3AJaAfiZbmMXiJtNlk+nRdyC6FzoRW2UqGPDnGlBrTdsBIp9U8Bj+pQRgOMr27dTrRO45VVaMvHpqvcEo+ebvDChkSxoUMVOOX7qsfO8HD8mQj4yUq1deXPZ81kLDj3R1+L+AA8rNS83KaWoBExfD1Wag7EcT8DTDeXEvwIcf+UU58vgzypat8DrBpkD36pFy8+cv4rRauPZ9c46EHNpkAPMC1LmZ+BddOre79sVQWk/7gHZYfv7K8qvHHqcNP3/Z+8nFhTpFyg0eLKA8nsiBhhrAnVe7Oo2zSOK513DGUCU8rtNJjA8HDKEeNxVqVuQrYYXpJACTnLp7GmSP2qVzI6VWm+tipxOf1YW1GsoJPm7p8vLDH/+UP+KBbrvxSnqRvj/eJbUmwxNP46Hnos0JQxwLQm+QdEP1CRhOrcq2QhhQnPuOQ48rv3liuxYOVMzR0XLNqo+XfZ+N4TC6u6j09m/r3kxIkTNEptmhWd5tfATHwVT5smPrv7W5rPr8rbS///SWA8rr//av1W9hLtqb456V/TEw6lEj4lOpKZY+W2rVPYTc+z5hmgReK8cwLuELNjMhR1WfjN9UlEJWnYd3EhgmutQaFXFz3exXO2N7aTUQT2Px+88sD/33I3wJwp+brvskAfZGRxHAjA3mgGz3SUDJQr4Ud6nbJDIzvw+g0DR6LQzszyGLPlR++vAvFU6gAm10tJx6wlHlwP1fVQP0ZjOD8HSbyfbfOp3QVMyDMgXgNJWwTdtuUDxGy9FLziYU+Ny99yinn3Q0NxG1OOylByGclSMOMID7ULdLpO006DSxZ9SrEt3pLN0EmZt67/obmc+M40NPMi5/VWVxaDqGgTMm0q8NYqOp5jUamgKI6YhjTy2PPPIoX77Hwt3KtZ+7pKOb2LVMnQZOCzbUp5sP5LoKqKc+XuvDIN2KTo3QmlLOPu+icsd/rKdTxMT1yGg5cP9Xl9NOXKzMhj1whR2auMf2LHRqZC/xM6BJ+AZpYMhPjS0JAAAfk0lEQVQMiuNOMe/khSKbc/7HV5Uf//TnZd7keFl26lEcEDA5f6H8Emi5UGrgb7jhJFUt7hu4sJtLcuiPY1xpkOZd4z41lkQNMhiubLxzjVRxYsZOaij5Vq/Rh1wshysV+pKOqCcI32RgOCGqmVIOXby0PPror/ia5+2zV1n56QtacZJugKpFzX6n+VCRRiIlsDX0+NQbqHZJ6j419xMwH9e7+oZ15TOfu46AO8wJWPC77za3rL7mU05xNVIy7HOvcrG54idJ1eOEBqwgQYvCpkdHQwl5mIPyv7/bUU498yNlejBdlhxxUHnZS19apnbb3cXLYt1FCOFnCMZ0cbM1mk6klLE2sU8zhkzdYE3+ffOGm+VHsrRATgfiHbrEPjCSctuJjIeysSOdMQEv0Rq5/GScuacQ3vnew5awoSFu8vV/t1/50JJjKrbYhEkqloAAUkpIAIwj9JhgQQ05Roa9/p+q6ibncqHcomX9hnvLWedcyCb2uCc4X6gRWXfjFWraa2RJAEJ4OopzmR+lA6RwpI/ptCayWWIsOv8Lr3R0rCw69jT2Gnj1q/68HHboO8vcBbszhYeTK85xvFYtpMIObZyKnCVk0TAJSwL86+88yxXeG9z3zbX8FXrPIWPPxvCda9yMrtjZ5MGmAreeCg1uY7THtJlsJ+ybPq6Ug99zdPn147/h3z/4/kXlzX9/gGC0CIk3UYngnTwFlCZGRRobwUHnRJz88F16To6TpdcliTjZP37oZ+X4pWeVLVu2qlQAzSPGJsra6z5VpiZT34F0mxhzCYewcQEH0BotqjcqXOQ1CS1VITWQHcNBKavXfr3c8ZV/L3vvubB85NxTy7x5uwlssauP9waQEIynTeV6wNywqLmx1rVMGrqaXGYPKLAP373roWYxz8RTVIlG6KI8nR5YirAF2GDt4OWNVPgwzNbrPVvVLJZy0LsWlS1b1J3qqs9cWPbZey9VHVfEBw+A3Cds5TTDHGgI9CqPPZGMxHVTMNN/hY7Ihv0cEfEM4bNDF51YfvvbJ9i6Bu+HQK694YqyYO6kw58W94jmoROJ5yBpmQ3t8zvZuaFNhfCbXMYqs13TZduO6XL8B05lx83LP72CHbFzAtPNpYHd/VPoVAYs6E8gT38cTOd+JWTY4FGo2bUUBgmMlydQV79h2Ex6V5bI0BWS5faHcB6mT2S8RDz8W99+OLtk4OtLt1wF/EOhicvpIf0AKuSNjjATj+w7oS5TWGgOfO3EWZLO5vFGsDDFKP3Oj/rAmeVnj/xCADVY+6NjZdnpJ5S/fNmLq2mhGvX8kfRxYKzpvrOMjw2EJ89IoXeZYU4OUlwIi57a8XT54Y8fZq+jl/zZi9zmxT0FepSs8zV0shO0yBZnM+Wdq1AoBy2ReQRv8MA9X7Tn4o7PAl913P0XvFg8FSVOkwCtrIBOUq1hK76In0HZeMvB7yvPuGH8ujVXUuJB7CIQPYPpAsj8K55EfhOUS53I4dMnyVRAGrvVTIGeAQKBIlZlOqbL+R+7oty5YSNLEXDP6NP3joPfUt7z9n+UCLsEnTNHOFldNrKNbJZ3my+GRy42giPGw2DghMbG/COyETjiWVCe2r8qpJph9sTraS8q1Bwdq/ZVTVHnred+IADspII72vgNYLMBepunlUvVhvo+uVxEg+35wP5Bq+Pkc44b2bpjZ3nbu48k7xS5wXVrVgnZgYogVAZPE6oCQDPQEBGAuXFO6DUcUi5e9Z3thOD2+GAGNXDSA0KsvvH2ct0X1rHQB/cDxOrFL3pBWXHu6XXVakhFdvwz5sIKzosHW4XGEB1LDVxPEu+dvB3OGhGKxD6DjI2birQEDanMCKhSlQ4F4+SYLsOT65Si1sYV1KFrbvrGGp5temUu3ORJJIWhEZ2l3lo1U41FrV4jmTk5lhXe969+/bvy3kOPJcVx3vypsubqy4F6skwAoyLILEDcND7J1mJVnfHdAQcd0MfLq/RHkb6YkiKpCuUEqKSSBcXZuPe+B8uKj32GM6jpWIyUMn/u3HLDVZfYAfOpS7bEnnCgxCGL5nWwP8LNZMm61wF2GQG/VF9YjQHKTVa29uvtX8IifZZAiFB5+iwVnkoNEUOnUWET33XfnTf6sU0/sIcYej0uBAmUa2y4zwh/KPZUy3SpBR5H3HOzDz38i3LsktNIcnrFy19Slp/xoYJS9Z3btqg7B6qdJybL+DimxEqINE1eJ5PqFNsSSj8x2MYLkqOik8ByOpYL2rmCMD32ePngyeewWCjwF4pyv/iFy+UlBFZ05Tdyn7T3rp2s6rWqOYPlzG60agCqa6fq6qZUUyWV2yeU4wDFNOA5ND1IczUBznPduQfJuYJrq7gzjiZxa5zOzetvIjuPx9cnETcCshJ+x2JRs/FiWwJltYd0esYAQ38dbPD3fvBfZekpyzlq4ojD3lne+uY3lB3bt7AdG9TSxBSaMKBKzF0k2KNQqR84TyEd5wHAFBehON6tHoyAPIbPsFOyKKPhFR2z5KzyyKO/MuN9pswZnyxfXH2ZVbO6hijOw4lSTMnT3YEpGjXsbivRhv1J5WZLoBKWtVPtMK16qviL9VdX96qMjVjzAQrk8ACwMBZgDUvTQoDFrItsZhwBOiymSuCmpHKFh/Ir+sXE6NnhQYRC51PHf9MD3y3Lz/4YsxAXnHtKAY3/6afhoIxywvrYBCbOKVYNDIiAm2rSjpjMSFvcUEDjMeMkslxvu7pYqTJNpxt5zAsu+my5e9ODdIJwElGredO1F1H1MylMeEyLg8Q2VTdyqPERSJYT5TIpwVRk0Y/g7TUgAXzXpjJnw4w9608CJC3mONMpuIQyem5djaBB17E7760nM9ARXpwp4zXOjBudoLxmwfFQzdXu3S8qhvTBmZkpd92zqXzk/EsLKjZuWHlBmXFL66l5uxGmw41q+jnojJpGRwSHp8/OQJCfJGnjTdafxenBq7mRNUepkvGrrr253LD2yxrMjWrnsZFy5cUfLs/e59lVSBAqseIbjSAcV7JMgP3xOHDEk+0HZRRV2HbWspmKAGwWbEMD2yF2DXqTtem98oaiyr4GVJCM6KQm7GI3I/9Oh1DmjSkwqk9nGibArPYJgGRWpK5DVxJMI5UlI2kQMTqlo5ZAwr/6tfXlkstWMSa76tJl9Ggn5+zGZgzoawCoLTQMuu0UwdS6hA7p9iieQYbTxVkrBjnwJnbnNLksNaN0FwalbLz3gXLuistZ64mC3KmxsXL60mPKa1/zioqsIN0mIYbNFAJFNW12P+5X68GWLEosMxXonoKkiUoVYw1ZE8P8cN6mnHGn4ggwhOcT0D8aSJvfTmUEQuGPHEJdm06LCV2DERbdcG60SV10//saknoyjA6Fbeb6+wrx+XV8r/NwN91ye7nyc6spiJetOLWMzV1Qpgfj5WnQBvFku1TQGmI1kR+XrEViZ5caVvQofXDdsAGGJSpJ+VLYrwEnDSw+7ozyuye3svyPk4He9Ppy9OJ316wP2uXodjSgtX6lS9mI2merEJjdDx2PB3vCmrYI8amntqqRZMII27icNh6innNl3rDWDiV8rXgoIAkuhTystJaplrHrANrzZuKLfhHWQfGWu2Kgq0mXvMZ7ghEm2A06wwWBA+HY6s677ikrLlxZJuaMlDNOOaHMmz+XTsoUZm+OjrEhoaBC5Ck1T6XPrfL+HM9VJmFQn5rgdnsVG/bEvoo1AQaMlEXHnVwe/sX/1DmZf/z8fctlF39YGDHL8NQFGvCdOlOLXoqFZek9eLYQMpff0aO2GsQ9M2VlPhDgyJ2ceiCh7oGYoDh4M70Ez4+Bx8okA3KWTojTKXOIg5SbFIMTITaBOgSDMth01006WwPR6RMWaIwUHkZqIJ6jglXJbDYzniRDGBeiRqfD5mBj0fH/sccfL8/e61llzpz5fEBQH/G6Flca3fGAmnY0Wopu6D5oMBIjxlvUaZQtSfCtxg9nfvjjZcPGzWovMxiU3RfML2uuv0wNK5zPxIbihBIBqn6CEtGIgVW5JYdQSBA/qL/V6vegQ6aA+HY/8Y5lX0OO0UkjtAn1icJiOHOoO3UFGdkKGIRQSxj0mcnkUNluuutmjlzMh/RoDq0hJVthS1W7Vhs05Mx5ClDgSAh/pbSOJzQn1UKQkCfBMDMuZCwkVm2fx7WCujYNMoNxwlCom+Z0RFJL9JuiHnWRsnLV9eXaG28jCI+vufPnlNvWrKzjg5FD3TWN5hbKW1bUiTnUMOlUqIuvdBBhWNNtKtcS+U6PB3FapXr3od00YZHPEpGgE4bRVeiysusZghLQYOjRrqFvyrKQVRkiNh5x03qlwKjHpczr96yZNPNgqFVMupDU93g2FeiMnqUZoRiC/GqoI1vQvDobcT8Q46tZdEP0WRfKIydl9hcYCDkSFLxAjp1Xefe3Npfl511Ytj2F2dMzZWJqrNxxy9X16VnhhSGnLqZVkTL+TwwB0CJ9xryZwbC7rFFOaYfzyncIDGkaKaq8wWLgVMCpWoaQUEvq2vwn86MGqEnl4QrDz3tlfIUns8f5hhgDuTEvXnrWZCHjduNnSYmAhhqWWDiQ0gKygaaKMOpotcmiGfJ9UjXWOEAVdHCHq2CbUe9DIIc7gbEZkh2uvI62yQE4vD20ajv0yJPK7554kuoPbchvu/nzHBGF0l6oWJxOshzwsATDR81ymCgzI9YglRYpL7b6p2EJsPeg1Cu4QNIQKvpB9CxBb+EH/Q+C/aYtWPNlcBvRLc4C0ye1NZMzyjZtEJcH77lVBzILb4MuaKrLdhO7deVufY0TZ9706Rk5SzraxkadfYCbjtZnPVCs1m7JlDsY50MaJ2aE4pyqVb0u3TxlOCsURrP24oSlzRlDB8SurKp+phz9geUc1ahM0Ei5/NLzyp/s+7yCe9+5fVvZvm2r70nsAdJBMEVigEl8hjQJOQ4DAdSynbqAeVLZ3w47UdIchEJmCQCbUs3KVSbprfSeIJ9dM+In8bOMAjWEqpTBA3ffTktcrV3lmghqoiPD5ojq4RZ9ELqgHB09BeIz/tulxHgzsIVpQAyPjYF10kaS0lxb0/lUO0J3nA12R4jKJJBOPIbF2sE5JdA84+zuBWoGOpLUGJFtR0GClio856OXlXvu+zY3Fx7gCe9fVA583X5sFwNbirFSWSABBuC5mnXu8AdCjXvSDJKW/oppUNynOBmThXRSJPjxD8JT17p59W17BeL0vSWEiePzZI8lSDz7/BwnUL6z8SsMTWrpWAdg4y44+oIhhjZtCPXpJFHi4g/zyeQNGTusgTddbTUzlP73zTCu0+s5prC3qU7aJvbNx8I52LF9G8siAAsmbIEdol9MvMAdlvk50+Xq628t133hNgb00IYHvu415UNLFnMztzyBERTbJBxsjjxWBmzX4nQcW31aqIOn/h5PlgJoAUe5hGJWpcGqVkkJXx5mFmLUHFJg47KV2jx4u9oTlvy7+JnLv/mbt7KnAaWMPUJz5MON7WVICz77q3m5bTNpB3rB6FAh9XzTJjb8UVdNoM/NsPvumMn9DaTCFZNhzrMlu9Y7asF79awLC9f80U8eKktPObeWGbz4hX9UPv7RM8r0LnS43Cqb6Rh6bGKS9hIV1zp17mIWWmTnLPIzOmBenCI9A3LCVcBIIwXZLQTu0G4SRmUdBNrHDIXMxkehoIjVn5+J0d531zo6QJyeqtq3yhSjcqhAgi4e4nGcHyETuoEZ28yA8tlM/o3T3pUnDbbod3kTFUtkM6mmIjgOP6Xy82F6N9QyYy3bzKSMaijVCx/qUKcH5eB3LmJrNtzVPnvtUVZdfgH7AD219cmagYCjNjoxpdNpFjrrRqClsJk109REWybH/zmTwfCkNhNGmKHYE9cQwz0NOVwWEniUl02DDm08sjYMvXJI4mza1A02rb9FhC7uSIJbbFCT0JoeI2CvUm2EKqJUpme440FfpwbHfla8r49n42BlKXIa+Ag1Ae0hrdSvERh1hpS6s5ag/ZVzFtQJjkJqH5t3DXMyWg478oTy0M9+TjW8xx8sLNdfdSHTcdu2oE+uCj45/WAcXaWn2M6lTx6w3HsI6mz2Ldl/lDEwE1RL7hq6pjpYpehk/2V2ZnNjpbla7K5io8ZYaKCIw7yczLaoVqvs0e6jXz3IeKmudegksZYsdCcnp4Nut0OEqh7dBJ8ikIIjp9kCG9bgGi4YPovXUJwZAaNwEXoLxCVTALUTJmEfQsEPOe1fV5R7Nt3Pe1owZ6qsufZSzgDDPBVuJkZtTM2hUzXKCe3usJIZKV2rM2mCCJpPZTURCkN4TJiLHG5Rl1MM7ZZmVBTIWj1tU5QKgWmV+w3H2VJblMH7N9ym8gQAuO6kRdvZoTmUwgrudtBUktlm2PXwWWJFLrbtcFRkNkA2sZGw6AxZhVhvCzaLLfK/1ArpfOKNxbTXIEpR61mYGgrY5N+09kvlkyuvZXw2OToo16y8qEyOospru8GaEatYjWtObx42hHAfgsR+Mi96MuKonspUp/t4o+up65jp1QvtYMf+5GGTwJ3lc/BztBbZ0Kw3B/BgHRCacHyU0RW8UbQF2SdpTVUqM0hxL4DQH2cnp7lBdnYEJCgLTvtm+xu+0dCJkfzSnqgXgNqkZLF0EkU6biTgBnRXwrWzHXpQT8/r2pHj9488+lg58rilZdu2nZy0u+Kck8sLnrsnPWN8AQOFvUQ9ZeAzaQmvQXKsrt/MoJgk81Uj0oqr9AzSeBC5sB/SaIKesyum2/cSyQwP4vMYstS6Rf1isV2m8MDdOpkhVWnZpaaiy7GZMOREcZDRZ5X0mApsQ4IyoMw2ZuyBM9xFKpmVnuKP19LLMy7LT06JQ3hGVK/ysMX8k82ocGGYaxHfPnVlrxd/omA4voWqfdt7jy9PPPEkTcnhh/xzOeC1L2ejp8H4eJmYmC+eK1q1VE/Cwsj7E3td1dPYKDhFcuAkqC7kibrsCFjp3hJVGYGW8BnfTo7Sn62NTL+/9PFtFFE2nmyhSW+AKzzLzUPgzOyGe8jp1Mk7rclrAwDKmlgtcJyxCNG8mWpYhIwoS99WikGwy96zeXV/YncsOEkpWXa5IUwPOV8UOybV51iXDIRM8pkp7zvqpPLoLx+j8B/w2r8qi//lLZpzNj5JThIIZvBe6YlGYH26gKoRAEQym4fCZRPd5sVjEyjfHEvUt0j9+9iYJZAQDY0X2wYPr0/vVNbvMzoK17x/w60cH4WFlApVBiTjFivHxouizDoAYDUdxImlCmXcBLUqLxgwWPVQzd7jIqMRhpl+BA6yI1bFcWwYK4J2z4lzVVMz1mv99IyEJElLwy/EqM/+RK3HdgKUP23ZeWXzt3/Ce/zTF+5Tlp10BFn2Y+Nzyuic+VXFE9h32MZGS4Nx91mHR924POIvge6iQB7XVUMKQYAhPEflpl2NNjZrIuQnQhwtlNdkFeJr9F2g+ZoH77m9Okft6LfFE+VRl8+JAUEqYDH+ggprqt4xSLJUYtCYdJCMBxoVqeyKwhk94NCOVRvOQ00YrXFQYzOIqJhaESeLNsm7TxOQOSJGkfTeUm65/Wvlis+uZt5w3+fsUc4761h2WpmYml/GpubxnlgOQKIzEtcAKdDvFgO+UeaHIRwKo5iwtl3Os+Nv2kh3FXFsiusojddi9thLoYAG8wNIdCzErGGuEQdIGnqkDL6z8ctD65gfmg3VIqfQk50w7JEB88SmCBpTVp6MNjfuJ4DcldfHw8Vp1gnt8EraWNsax48YY6Heq13iuav2kjqVrmbo4/J8giMGtKukdyoQYcwvH/ttOfyYE7kxu+++oFz60Q+W8ZEJFsUi5QUhfPppIVqY9EPeKjtVowCoNW6kQ2ZojtBaPEs3jaD52IUxWs5F9lgubaGT6J61kriS2sRcoirwMWH+l6hd14FlcN9dqDVRaJJFa3wTHX85Oc170g2quQM30k0WkoLKXA9ubJ99caActkBUeIcJ0GALNFCf1swDGXbjW9qpF4hgtwH3haBIGIlcRQvgu7GJctC7FnOc1OTESFn1ibOY1Rmbu1DjlHfu5KBysvScgoLpQHMrQWxuB4AWseyh5OFxSRCYDNejWHUt6ZWrwqzZU7eDMU1HJslkMMfS9IYzrMYs/pQD8tQizozbLKJtwxS5CMxotBylYjlJZjLucW5EfXCKysU4lReEU2vVE4XKG+BxVqZFuLsDbSBQfmjykDxlB8cg6oaFvlU9Jyng0RI1kb1LpGhtgVqHghFeSjnkyBM5SRbnftnJi8oee+5ZRiYxV9s9Zgk8GHYbDMokWPce2k3VSuuTcTJ2thIOuTsLNyUaxL5DA0Pw/r6o1nh21zQjfoaiw/ZafHScqdhUnswsTg/rxaOidneSV+C1Im/dpIBnOTGOE9OF0b2FqjUXpVSLOtS8wiUIWW4LQ7pcsugVFMoBqIsYKjrJijS56/pYago3OMr12VGSvdTVbEpAg3qg5z2nnHl++d4Pf8SL7PfKvyj7H7h/GZ+cqszAuWjwOznJcY5gD07NmVJBU0KGKuh2K7yBdFxqrz/ZfKFX8T8UKrWNVnQQx6YC9lZHgRir5mtguHyZ9H6AN9ukuwWjCRUQ91Vko6NbhioflawAf7hOMm5UYi+iJ7EDLh0Xv7W579wgxpVmIaBUYifGXDwllT42zmb7WlTcbyBHhAkuUzD/FYuCKbiMo51cF6IkH+DmdXeUz16zmk7ba/Z7RfmHN76BwjkHG4iRGRMaQj5hxvvElE64vmSa5HwKaiT40nmm0jztK4eGIZ292Hj3ShCpAk1yLf1Vwytcq6sYpx6LvfVrB/dtWDeDh+HEdccJ2XghLQK1dTr1n37f2SKDDvl4bJhOrN6bG89jSULdftNBd/ubsVdnWXCqOBrRQ82hJWnb6WSpF1G0hZbYWXjPpjaCl5uoZgC/2LrtmXLJJ68sW7btKG964+vLc/beo8xfsKBMeho7Yr5IPl4/Z568XGGhScrjNUpSB2CAP8ExT+kl2G2o9kmIGhEyqxc8J+XSlWw5hclK8eR2IZ7W1I0rMt5r892ijYCnGdUKQ98gN2OPhvXi6kdFVCcGF0kWoKrKndwEcWhbpiGErZxjxH1aHC1HBIeYcNSTFwE5RszPTFlb4uM06q39cQFxWZBw3YRI/bry97tmyk7SPcGOTz1NzIhezaoVDMiZg+lG7Qo5lTl+NYdpU6I4UKc2taPVu07iwNIXu8rZ0z1dx122uT728nPClXLEeGed6sGDG788o4a0SccoPFCT1nSv0sMmruED2qui1+n6SiYcPEMZnhub0nOhGuQRhgEWLqmsqIwQmrhedqZ0rMVwwOvHJyfLnDlzh+JSfEYY752GMoDhHgU7hRGH3BzB7e0YQha931VVFs6w2yfBW/UAWPkXSh6HCpJrZru5pia0yxNVjMt1BB/ZQlLJ004a9BXp3MRUshu4CbWzYueesjl4cOOXZtB5isQlA+4KGOV+p4xOqiUqpmmt1rRPVca5WdyEmhMhj2nV0uGq4Omk2jinJukiPCxmYJM/mtZrLshZsHDhkFBF4OBbCjhoJ0cbZbuVheo8S3yO+qyD8KXaEmU3mrOiPnw6sZgtJmfEvFl/XtJyUaHcAEsVMh1JGIRZQflU5t4C1jk/FAD1i8+JV4gS38DJhqEkhJPW37//32aiqmrOkWV8GoCiI43WpcPqhZtl1nfsZ15Rpxa5h3hNQfkBsSCsoxiilVjSPd8ES8tGSumXY6L1/AW7NbbBUO2GlfaswpwE8VTZvkEx9loIVjWOjko1wZlxSQyWczJRaxIvFFqoZXUSo/dqnI9bE+jhPcXeCkumxQXdtAqj/s55JmngbGwbJkfnTFRVaa0mvYPvbAKhq1H39GC6oDbZCdKuZ3o2GL3oshAVkrKK1PulZsUIaNVceeBI7+zcIIeadoCs1FBhM6QJd4xuNlZXk+Ch8NRuWASx9t2R04E7iT+QZ6w2r0JofW/XeHDm7vjmU79JzJWNolRUFPSLqTO81X9P+qp+dgTdqhZcBvkKqktVxqqdoBxU4t+pY62dqw0dYjMD1fVoRDDMqv9r0rh5cthMLiTL2JySsfGu6ZxZeclkIOgsdBSInJx2atz5mS20p+mkzJsLANxkMEqlsN0A7xScToPEpg1JMD3JNnUgmK68YifCk+XoWtL0oUIEaUigwutNqX5FnhTeBL7kNEWXdOBWR8lAUPNGdDlJHUst0uLZSnMssy2IV6eYF93VHOp8b7PUbG+8A51VVUSMtaXG6ul2+xM2YepK0vE+JpjdJLZeJ1rB4UXtDmIV2BAkZyNadE422xQAcNUdVBWkWn97wQCxO28Q96kpEmaLW81nrjYbNtnRymb2ahJsp/BX46zEHlJwKhhn7WAvNqoOlnPUNZ0xZVh43E8PmWpzZffGxzHnxUBMvRlptuq0zZoDk1fTm82pijcaRycWmDfHRUvdf+xNU3E5yRKELhTpu0bHxnVs99gMAvJJ/6TqOvEccMwBNhO4qFNESVDXId2NEKzydR1dZXLUODiqXuUHnnzUjV+uoYzDiYQkOey1tVrnyEVV954+ZSbxuMEBw07WvBBIXTVt3MJ6bIyDah+qBsMz8e8urVQ2ScLN776z6Q5RLR3jKV5rtpU2052xqkfVEbl6SZbagTTrRvvX5+fZ16iLYPA+TlEgRB2mmTKOoeOct9zSZVVSmTFpoZTAjah+JqqGuniZgFJrUxQHKkuhEYaNuoJnh6OXqjNlM8w47yYQsdSut3FxuGJHZ8XL8CeSbUqRcTuxErw+fFIcagzbIH+yUIlR/w8zhPQ5IIcBxgAAAABJRU5ErkJggg==">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -494,7 +503,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1037" name="AutoShape 13" descr="data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAHcAAACfCAYAAADDLkZlAAAgAElEQVR4XnS9B5RkV3U1vF/l2DnMdE/OmpFGWUIogBDJYGywDRjbBAPms0wyIAMGRBLJBNtgMNiYbBwxwQQBEhJgkFAcxck5dw7VlevV+9fe596qHsHfS1o901P9wj33pH32OTfYt293BAAR4mhHbaCtv+orDENEUWh/Cdr6FrUDRFGEdhsIAvuz/gfQaLfw8je+G9VKHWHYQKtWQ9Cu4kuf/Qfkc3m0Wi3s3/c4RvszyKSTSKdTSGUyyGazSCRS+nsQj+u6/v8oClApVxCGEZYqNSxVa7jxHR9DaW4aV150Ht77rr9CrO0+H+N78CuGCAHufXgPPv/f39ezx2J8vwixIEAsHkcsiBC1Q4SNGqJWC41aDa12C4kA2D7YxDOv2o7hgQFUwzg+/fNpRLGEXdetViwKEQ+0cAhi/AO0VlG7jQghauUqmrUKKuUy6uUS5s8cR1gv4+tf+SzGR4e0tvEE15C/F2ltYkEMcH9vNJq6F38eRnZ9v95xBEilUmiFdYStGk6dOIZ22EZfXx+y2TxyhaJ+L/iTP3t1tGp8Fdat34jztmzEcG+fe9DICTfSRf2yRVFbD2MvSiGb0MN2GyHaeM3bPohqpYGw1UCzVkU7rOKm1/05kskEfnzbj3H/PXfhkx+/Bel4DNlsBulsVg+aTKb1PZFKIhaL6X9bsACNegOVag1txFAL23j9u/8ec1NTGMzF8c+f/hjisM+22m3sOXAYv3rgITxy4DiWGm3EErZZYjG3KcMQiUQCsXiAKGyhReHW62g0GhJ+PIiwsaeKp16yHmtXrUIUj+HTP1tAvc01iLvnanPnUx3cM9rCt6MQ7Tb/b6FRqaFaXkS9Vkd5YQZLU2cQa9fxP//5ZRQySSSTSQQx/r4pB4VNycZjMYTtEM1GU3rWarYQUuJPEC5/P2w30GpWMXHmlIRZLBSRTmeRSKXRCkME2699ZsQLh/acGBnoxbaN63DB1i3Yvn0rhnp7kIgntDslTO7OiAKPd7WWwg4iNJttvPYjX0C11nBaUUVt/izQrKBeKesRE7E2Pvbev0IqFUc+n9NLZjIZZDJZ/TmeTNriS1NsVzebLcwvLCKIc1HSeO37/wGz0zMoz03gn/7+Yzh4cD/uf+AhPPzYPpTqTUSxJBLcwcVeJBO8Dp8XWnh+j8fj7tptRE1amCparTq4n2JRgEKsiudeOoKN69cinkjgS/eUMFcLEMQS9u5oI2hH2hzOrLnvttnDVhWNWh1LiwuyDJXSHMqTZxEEDXz7v76GYi6NZrOJdDouTe0oSNg27eQ12m2025GES7tIzTQl40ayTdYO6wiCCPOzcyiVSigW80gmU6DW9/b2Itj53D+MKGU0m9o9qUQc1VoZ7WaIdquBTWtW4O1veAOG+ntsQZx59prrzbJ2bBjgLz/5H1iqVE3wzRqWZs6guTSNKGpptyfQxi1vex0K+RRyuQwSiSQKhYJ2XIpam0ho8fkC0gaauSjC7NwCmmEbC+UmPvn17+H0qbNYmp1ALKwjigUI4hkJIqD55e8mksgWiojT1MlYd/+nWU7E3eZsNBDWq2i367pXEAGZoI5nbC/i/G2bkc7E8e8P1XFmiRoWM0HQVYVm1gNtHLtWRwtbVdQqVVQrZYT1GhbnJtGYm0EAau7XMNhrLioM60gkE7omhcX3pWDCsOVMcKDPaS25meT+6FpskzXqZSSTcb3j3NycBM0NUSwWkUqlEVz6e38W0QwEYQvtdgNR2EbMmYlGs4l6rYqoUUVfIYPxkRGsXTOOLZs2YevWTRgeGtSLBrp5As0oxE1//28oV2niqBV1NGtllGYnpL3xRBJB2MTNf/FH6OnNIZ9LI5nKIJfLIZWi9mYQT1Jr+aJudzrhLswv4hOf+xoOzpTRbNHHxlBZXABaVZNbLI6I/wNoxxJIpDJIZ9LysVQPbZJ2yKBBmyAe8363hWa1bO8fciHbSCDEUzclcNEF21DMZfH9x+vYP91AW5stpP3vWC2vTTTpuj4iNBs11ColhJUKanQpcxNoLM0jiTr+49+/KkWRnw0bLraA3IZcSytEeWkJcedOpFDgs7epGwi4nSIgajVRb9a0VqlEsmON+DzJeByVSgXBRb/3/yI+cIz/B3w52gnuDwYHNIkN+TxqMejk0ZIwW2EL/X09WLdqDOvWjuP8bduxZcMm/PVn/xPVahMhzXezLttPvxa0GmaywgZedP2F2Ll1NYp5+lyakiRy2TwyWQrXHpTC9WaZL1ZaKuND//gV7D05h3gyi3gQoFmpIKxXJNAwCJBIZxBLUoNTABeLG4za6GIGmjagLVMtn06BhA20G3W0m9RcEy7DsStW1HDVZReit7eIu48s4p6DbYQxoCk/3ZSZpIAoFC/gMGzqHZu1GtqNCsLSNMIggfL8FFrVElLxCF//6hcx2F/U74Rtu04Qi/TOFFrYaklb+T9NNs1yk5tA+5ebMsbXAtotlJfKilMk0KS5MRNuAtVqFcFVf/rWqM2oOGwibHFnh7ogfzZUSKAVRphbWEIMfBgGC3X5i3bLBBw5oQWxJPqGVyKWKQIBTU2of6MlCJs1mRqa/aAd4tLNw3judRehJ59D9hy/m0E6nZFWxuMWJCEyX1+t1/GrBx/C3GIVSQqPzxO2pBmtKI5DJ6ew5+RZNNsxtLXTTbguvAWtc9QKFXrRp9vGaaNN4dariLVbCClkrVyIC4ebuPqSbbJOB2db+OZ9s+6eFD60PmHQVhBGVxBvR2hQ8M06wLVsVIGFMxgYGkEhE0c+m5FretMbX4u+Yt75aNt49UbNhNOJvGMmiyBCo1FFvVxVrMAvKgJjEH7VqzW9H3/Gzeq/h+0WSqVFBFe/5t2R7VZudpfatNtotdroycRkYqZn5y14UNzUtB0StdFs2SZoNhr0BMgU+xBP5QAGHtQYviSjvVZNG0I7vd1CXy7CjS+8AT35LAo9PUin00qHaJbDVhu1Os15HaWlEqrVinZhs15DIhWXX47HEwhDBhy2Efn5fLYHmYEVuP3e/fjFYwcVkJj9Mn+mNIUuh+/p/JvFCQ20aJZb1A5ekzlehHXFOp5+6QaMj41hqQH800/PoN1O6H0DcHEjDBT5zGkM9OXRn81ioL8X2UwKfX1FuZreXApBImUbu9XCvr17cMVlF+q9eR/6S361I258CtoFe863U5logKgQ9XpN/tSsX0uxSiyyYIxKlkwk5b/lixt1VBjAXvPn71PmRp/DXNDns62mRcV8UWpcm1Elg48mc6u6KYW0toEg5MZoY/P69ThvywaM9OSQZg4Xi4EKKC10L0gzz5cZ6c9LSDSv9A8MJChERs0UYDqTRCqZQiqZQCadRiadkMZxd8oOd/JBPkOEWrWGU2dOIwwTOF1L46u3/hIhcwkujswvN2cks9YJ1Ghdwgbq1TLSQYR0PI6lcglMYEdSZTzzknVYt36N7neqvRrJVAqDfT1yHxluRgZwZgsxPTWFeDzA1NQkkqkc5ubnUFqqKLg5dvwIVo2txHe/+x18/CMfQCwWaUPTlwbEDWgBWg3EYknlurQdDCDve+BBPOOGpyIZowyaWn+mbMsjfioNQQfLMOKSVbNVR50Yw7U3vj+iEGmoFIbL13IHu8Scf1cKxNzOojUKmoJlJBhr1fGC6y/Fjs3jSMRjWCrNI5vKKSBoNBtgwp1IxBQoJXlzhAoapFRRhBzz3GRS0Z38V8yAhg440qZ1sGCIGmf5oCklNw19FXNCS8+AmdlZHDx8EpX0CL56610IlbrQUjYUCctnKT9nAETLUpNwEwyklHY1kIi3MZZt4Krzx7Fh41pF1unRnTh2ekKWJGwyep/Te4yNjeHI4SNYtWqVfpcpyOTsPC7cuRMnTp/C7MwsxsZWYbC/D3v2PornPvsGpBMGWtRbwLe/c6vee+f527FqfBR9vX3S4jt/+nOsHBvFdkbsCcrPfD0/y/twLbjGfHe5TFqUgNF1Uy5oqVRCcN1r3x9RmPyAsxE+PkMmkcJAIcCp6aqZOQrWmQbu+EzQwptefD2KmUBmiClNPkshxWUuFFy4FMv2o4v95OsYtS7LlZ2W0XTSzCYV73Tvx5fyaZG/jpQGMSSS3LGM9tuEAVCuVLBnz0GcaRXxPz9/GO1WXUFiPp3AxWsLuHvfFFq8X9RGWGMwVZOQGaRwYccKIeJRHRdvWoEd521CKpXARK2AX9zzMDZs2IRypYapqWkMjQxh5cqV+N73vod8Po8XvejFiMWZf4aYnp7F7PyC3n9paUnPd/HFF2NoaAgjQ3149NHH8OPb70StxvyaoE2g7OGvb3ojfnDrj3DrD36AN7/5DWg1qrjskgvRDGtSFH7W0qhQG1v5rgIwBq4WffNeCqiu+4v3SXO5q2WGJUR6nwjxCNi+YRiPHpqyFMB9cXeg3cSLr92BJ21fhd7+fqFN0ipCegw23P9mAkNpDvNLRqsy8+22QWj02w7l4uWZs8lvVCtaKJpEbiy9xLJn8IiZ7C5/L+61OpDmz5dKOHLkNH7w6AT2HT2rGCGfjuPJ6zP46d551AnPcbu2moJJm82qnp1W6bzxAuqVJWwcLeLSi3cgnUphutmLA0dPYmRkFPsOHMLiYglHjh7H+Pi4rMVA/wDWrF2D06fPYHLyDEqlJSSSGQwPj0i7FxbmsXJspeKKI4cPWcCjdzIlkEWJAedv2SxwYv/+/Xj/+27GY4/swgXnb0M+n0HCWR2uR6vZlHAFyLTb2iQMGJVtR6EsTHDtje/tCNduRPPGZMAS53iSUbJFnxI+N0KrjVy8gXe+7OnozWXR21dU5CksmiAkI2QXbBHRUpgf2gPRZPA+9BGd3+lsLotg+W/8DP2LUG+lCUw9OvvLmWb/g2464v0p3+HUyZM4PVPHF398P2qNFnozCewYaiHMjeCBvSeRSiRQqzFYo6ltCi5F2EBfNoFsooXrrrkWv/38FyKdzcnvl0oVHDl8FJ//wheQzeVRq9eEDDFF4aoWewrYt28fRlesQF/fAFrtQJo9NTGNUmlOqQ99Kn2th1cN+LD3ovYODw/jJS/+fRw7vB9XPekyVBcXUOwl9p7QBuXv0Rr4oNC7L64989s609Z2iEqFqdBrbhYszcUXRBcx4GAyYJrMpNl7346za4a4evtKPPey9RgdHQEzC2+uqZkyG8zThKhYPpgIYiAowsBAvjaXQ71uqJBezN3PkB4GaIax0td4M++B8+Ui9p+XgQ4sWJJG0DoA2P3obpyuxvE/d+5CMQlsGWhhup7Byfk66Coo3EajgkalgkioXF3mmwWJVStXM+LQZqfLyWbyyGZzaEcBFhYW8Mhjj+Kee+/Ffffej6npaaxZvQqzs7PI5HMGwsSJmScRRDEUi1kcPXZYKQ7jCgZUyo8ZB8g9WRRfKORxy/tuxt7HH8H6deOIR21ksvbvwhrcl98cCqhkuUyDaZ4ZoApyvfLPbpbmCvtwbre7+/kz8580WVo4BqBhiJc+/XxsHMpg3brVDv81oSGyxFwIlSss0AIEMA2uVqoK2ROxeBdacwL1u9C/gMFyVhmx53MPeK4Cd/7mn1vBRtzSAqYQu3Y9hj0zbezeuw8rM3UcKqVUZFAkHTZRLy/JHDNto4+77uqr8JIXvlCRev9Av3JtVq3o3xn4qdDhChzcoI88+ig+8IEPoKenR8I8cOigpSxRHP39/fLH5fKSoljFIA1asACJJLOCTEeLqQCxRIRnPe2puOKKi5BPW3GBPp9f7ZaBJAbyWAzCdJRuyG98Po9wCKbJT3rNuyMFIsJgfQnKBT7SKvMLNCZ2B/PFr372BVjVn8a6tasdKN+WJkZt213LzYV7Mn3z1Q+lJ4pwl0XGy+xuR4MdLGc71LTo/++LppsSUwZHpIYmJQDOnp3A8bOzuGvXbqC2iAMLcTzj6kvxiwcfRbVSQRIRyvPzCkQG+npU7bni0svwohf+AQrFgl0viqucxjhAoEqlqjyVQuYasWrF7KC0uIiTZ07j5IkTuH/Xwzhx4gRKi0t65HqjbIoSWnoZSyakwcoSGApKkVt48R+8AFu3rkeB2i3hJs0tOQWjVVKWQL9L96bc1/ytMAfluk1q7nusQhlZqtFJE1xqQbBcfqFTAVHqiz9/5vlY0ZvAxg3rOr/HB6gsLcpfdyoYDvAW1OZqxXyhSsleuFsL9dG0ic4n6su1WYFZu6Wgi1GxnpsP4x3HssBQgEk85oI44NHH96IVJXHw0FGcWmhg/fgI+gZHMDQ4hIH+fpXLUpk08tks0gmLXlVFisWQSWclWOEibZrUDGr1iqwCNTURTyKXz+udF+YXUK5WJMR0NoOJyUn873e+I/NdLptw6Q6IMjVbTQcEGRAR1htIpYEPffC96C3mkWIVLM0ghcBJgHjCNLQhDbac3UqEbTSoWHrnuFxGjMWTy155c8RI08phVrf15tTySvu7yt9Uf1NqPP+SNbhgXS82bVzfCYDMfDexVF4y/8cd2Y5cGhVqp+VUtG9q9zIg6ZrabrTk/TB3p2BM909W2LY8OU7smT+QSfJglAV83nLI7MaYPsSFjz/62D5c94znqd4ZEg2KMfFPyYQrkg8MpeO2YcZP4bXCpswysW8GUbQcNM+EEmdmZ4QMWZWJ3+nr27ywW+iYolhu1Pn5eUzPzGjh77n7F/jFL36JycmJjmIoR63V8PZ33ITVq1ciGQ+QTlC4cYQNCp0YssmCMCdjGhYMVCgJQ6WPFDTXjvdIJTMILn/VO2UBKWlfrPaLaz7UKjD0oTIeQRvxNnDh2j485+JxrN+wVqaFX1aesjSnWlmyPMwFVDQbFApTASbhUjiaKifg5f7U53DeNC9PlQii8Y2a9aYWk7iuF6bcyxMjam3IQM8yNTWFxVoMVzz5Wkrd6sdErOLJTqFCG9j5dpo7skAE4MQCZJIZ+U+CNY1GTSaQrsj7QAYIlncbmtZq8/3qyhL43pVySegU14km/P777sMdd9yJo0eP4PTp03jubz8bV11xuYIvXpPlVxUGtKGbiDm4kuuYEIBR12b05plC5v2WymWkkmlq7jucWXZUFfkt+5LGsgjggiPT3DZiITDe08YfXb8DG9evljZ64aoyws+HLbEQkuStOF/LQrIvIFh0zntSQyzlEfzpvmgWCSj45+hExYH9XiyKqeIko+wDCqVs50o3csKVBiPA43v2YeuFT8ba9RtMKMq8VXMxN9EJ2ugDabnsPSw6tY1ubJhIQvYgDYVJK2csD4MBCZTwegycmNYlYsDi4pz8Kl0YNwo/t7hQlmbPL8ygulRCb69Vyrxwk9xMzZoqUnxhwqD8A7GD5QEVn4XgRa1Gd5FCcMnL3hYpqPFpRGdtXKmMILaAZGfi3L8n20287UWXYXSoz6r+QkYM1xQUFllKxPCdL0wfQw3nDhRI7gIqL0wrl9nFfZ77xOi5m/bYxqM7MSjTIEtVaFx6YWmYIisnNKYacS3yY3uO4dnPeyFSGSuX8YtuhNiuT/wkaKFBDOQMaWO9VwGhSn3UqrRlCIClHwF/HpMV5LuSXCAWi6vNJhiJAsqN+T/fmbynZCJtkC9YVWrizKkTqGszBDLHRNJIVyLUmMkVkMpkUa8sdqyHXy8KmrVgYupBkEJw6cvfbneUD7NgyV7YUhmmQh631ILK5wDxVh1v/8PLMNBTEKTmgzHuMOZy7dAS9kadrAwjqFFTqAlaECfIrsDMXEkrl2HIv6a5bjf4KNsjVRTycs3z5tlxy0yAcZW6cfrMLNqJIp507XWqk/BaRr2xfNJvKmqpca9oFrnwRLIsN7d0LiMNYQ5MbVlYmNOGYGVLLikRV+GABDdbO7uO+E/U2MV5LJZKKOSLqor5KhEtAzdhfalqOTsiLMxNoljslRKSSDg1cQqlhUkpAk0x34HPQDM+PTuHRJxMjJe+lQVJRIqUCf/ZTiZ4YDbRgAEJgQGHUg0D3d/54iehmAywes24gwctJDcQw1KiIDKckw9v8KQn2PlF9KaXv2vWwtNMfBTstds2giX+ntPl0ymad0uXvHtxj99JjR1MSbZGFOHx3fux8/JrMLZ6nYu2TevFjqTv5KK6gknUpOY00WjVRD/i82kzxGLo7x9COpVFs9XA3Ny0e1RqcFIuIpW1PJbFBwneFT6MhWk0GmLPjHazOUPCvKlRgMRiRqOlfJi5uWHLdVSWSpifOo2lpRkr6BO1Stimqdda2nDBxX98U0Q6qWgqFK72tmIw96Cs/Bthi4vCRNvAhQg3PudCjOZi2Lxlo19/l2M1tBgWPTc6YIW0ZxkYYYFSl/1HLWHkKhO4DG/uBDhOuKTIEL1a/kXrwM8puhZo4nC1JwjX/LMVuh/Zdxy/9dznI5svuHeyjexNsnJREdaYP1aFthGkp4vRs5JBkiuit6df6zUzMyUfSHObSuWESbfaoTRVbEQfrFGLVaJz5S3lwA1VcuhPqX1KcejXEwmkEibwIGb/xo3E4KlRW8Dxo4dQLc3Jz/f1D+satJ6yghe/5M1i1lC4/uZeUy0ns+zC82vFjxPJIcQ1O0bwlK0rsHXrFlc4aCl55u+1+AAMrFotwWvM1Qj1KZ50tFWzEA7JCq2Q4Ivsnib6RDzZ6Ddd7T9HwmZqHGNCEPoT/tl5IAeEzM8v4PDJSTzzOS+Q//QbWoFdRFaRxQ9pgggqdZKtYgQELTaVIp5Af98Q8rkcZmatwEI/zZJpoVDUJiNdV5uVVonmnUTEVMoi3VYLibhxqfm1uLhoOTJpvtwU+ncW4pNK4ZjiUF5GE2qhVl3Cwf2PY3F+Dj09fVgqMQ01GDK4+MVvEk5BtqACE1fM7vgdnzcqXyVNxVILCq4/HeItv3clRkZHMTBgfGdqnZCqiIADqTYtBQUeOmvW68voJLb2hpCZ0P19PT/a57ld8+tAlSdK3UX3Xpr0l6KqSAodw97RUKV+beaq8zh84iyuu/4ZGBgYtjRZvpbmjxvUKlwKlEgcbDWNeN6OUGelK5lSmtOpRzNflZnkBogbdTdL6pB3bfYwXCNPi2FcQoF7mi/9Lcns8tuKU6x4kkynkE5lkMrkrPASMpBsoV6v4MD+fSgvzuk69NLcoMFFL3o9QwhEZEUQNJBZ6lR3WW+zxfk1X8laa4i/fdUN4hytW7+28wKMHK3CxEXgziMXy/vgtnwwAzNPFKfgCAZ4U2vafG4aRH/M3G65ue6IbDlw0XUQekHDpc/9ksmWfzWG/1K5gj37DiIKElg5tgpr127A4OCgu58VIDzEZ9fjolJ7LMUJ4gxyMvocfV2rEcqSNeqmpboPImcdgAYpPUSamnUJiQwOXscHlBZcJZUedTnWvCchUJLOs7KGYrgYiiFTffLEMQVVrXpN6FdwwR/cqJoT1Z67k0TsA0dPd0vryjWJUHVN6PKU5JaXXougXcO2rVtdac6iXtYTzX4bX56woZTItaeI3OXyyi6nyQS63BfL0DpfawFXF9p8otC6Wu/Nbzfy9puik686dWaQQ2GTBksTWa3VMTE5g0qlhgVHMS3ke9DXP4DhoSGlfUYOIJCQknWoN+rIZXNiYLLa1aw1kS8URKy3ANN8IHlP/N12ZCkZW1pUCGAC7Kyer29TuD4KpzVUoElkLhGXcJlqiQoci6NeqwjQaNSbItrVKmVMkgR//gteHSkBpyaJdchqSlyYrUyh6vfEWM35GhzJP7YUyd34nCuwsghs3bpVHQR6yEZTjD4+VCJpEaLHpgleqCYcg3YZL8tdL3RLfTZ2Xx9oeYH5mq58iRTPAx5duNGbbtsQXdFbvODIb8twaG+z+VkFLgpkmMIQSkyojivz17bFrzfrmJmZxfT0tEjgpMSsWr1aqQwXP0PBtppIZjLa2HH6Sq4tTXQU6X3FmVavUoBK3Syc0KhUyoAKx1zhc/B3adKb9YbRaRy8SBK+8OxcQZrMtaMZr9Zq6CkWEUQBZmYnEGz/3Vcqx+EuY7jeFuUjJXqo/ITrYVER3tFYZHLZQQDgwrEc/uSZV8rnjowM63cogHqdddKGcjcJV5zgCG0KRyprQVHYYOTpfG1HsBLPsnzT0hvvm01QTjTOny4XrBduJ27oFCh8T47Vn31aJdMp8ME0Pc3WlnQajUYod6HiAIvl4mzxO4sFBjHy6+ix49izew82b9sqZgbf0PjEMcGrPYVep5mEK7kmZiVJjGMaxPfiz9LppKwHyW0sJPAzJAlmMxmhZPyZZeo09QnlvLQUbLFhlMzfZdkxESRRri4i2P68V4jayg/qwblzGYmJLEdz3MVuzX+Y6WGFgzsm3W7i7970+6LAbtiw0VVTrAjuuT7aJMtKgR7BUiRKaK5OaqxXNa+JxrxQeuZyU/8Zn654c+XTmyf64K5/dnixAyi8b7NQwmu0gRmW41r0SuSIgZFxlRgZ8ze4vPSxaYuWCS86VubMzBz27z+IK570JLtWKq51YqtModAjM8581mDZBGJJgy/LlSVZLU+WZ6DH+/q4gxuFJAGiWvKzDo2jD+YXhcvNQVdSyOdlHcSh2vbclxm2rBezfJcPRqaiAhsXOT4xkOmmMC185FXPQrO+hJ07L3DQIfFiEy4XizeKBZbndfyiQ6oyqZS0iFxb72tN84zyQwK6Uip1QXRtrU/bfMDkg7Ouj+4iTd786rvCRxY5iKBZZLs8NZPPZzBHocUTyjsJIugzrrYsLXepi6FbKbd2AaqVGnbvO4Drr78B1RohxhCBCgkpFAsDpu3tyNYkYcgYUS9qsHhsrmnNWyoJ2OHJ9KfcLHwmw/u5powZLP+lkHldYtYsagS/8+d/GR08OSMdpW+ieZZm+OYmn3g74prw207QY8X3N//+1RgpxDA2PoahoVGpGyNBmiQrAIRqWvKRnzZG2Das2ZHVqRRM5K0obULkC3iozufZy4O5bnpkSM9ysGP555ZrtH7H6Z9v2zB/fq7v5u8IWWIQRGy80ZQVD0l7SRsZUBvVce5Rvt0AACAASURBVJ+kzxR4BDyyey92Xnw58jlWdyI0XarHQKhY7FNflFwSsXgR3QKlRhScXbPLkfJKRMXLptMq5zFr4Lp0SjxtA38y2Zyux3hE6/Hhv3t/9NXbD7o2CiARTxnMGCfDwFWGhG+6PE3+MjCOkjNpT9qyAq95/tWYnJzCBRfs1NIRIvMEaj4wheuDB2lb2Fa0Z2VCa4uUTw6NOsJVoub4AGt5arRcO+1xzPH+prTHC/Ycy6Mow2izhBKNvdEVrv8dBUW0ZDH24iS1+ZSzq9vBqES6vwvSrOkMwnYXy3Vcc91TUK2WxNW2jUgYMoVEusdhyQZu1BtVaR5JbRRwoJ4ti6TlltRaY8wSghuHjxzCyMgIEklWh5iBEDWUzhsa1nJdg9/79ueiv/qnnyH03en0u/IjrEYAqXQM1bp1FJhZtZ4hARmCJUNk0MSn/uqFmDg1hQsu3NnlDIkr5CggjvBNVEV+goxBlQId6WtZIYE72gdP9D+eWvNErfWbpZvmsLbpUq4n8K2kEYIlfWpl373Gd69t2YDfMN6ke39sjVu/HuCZ8CxQa7baePixx3H905+OVJrr6ciGDlmKx9OuWY314YKUhc/BlIgpZLlUElqmNhP1DJkVYYObqk31Kk6cOImxsZWyLMQxtdk8IhvFkCT/6vv/9dHon28/hb3H2UOrBgeXWFv5Kx4L0KJd74AKXXK4pUrkHcfxN6+5AT2FHPL5IsZXjcuMMQBg7XK51tSrS9rxhWxObEj17Wr3eX6VtTF6HrJniDzR5PLnvjNuudYZsvTrAvbCXc7U8KbRKLbc7VavXf5l9zXNpqXh330VpnvfcwEXtuLc+8ADeNqzn6kuQW+dvILQ9THVYr6bTOaQK/Zbg1errjUnYkWesyc+KHIWeY7tNGyxsRbNudk5EfiowWKfOtYMGSZMKoOvfP7m6EQphy/f+nAnWrQw3UB0htwG6Fg1xptJFbjVcmhoyxtecCUu3LYOfLHNm84TdEfnTmjMp01ajHbLismOikKap9ISl9tQu3xqIA12dWFvfhVoeO2xhKkTpC03p0ZmZ4pjLsT6WrsBmTd7pv2WilFo9G0+wFq+oejnaLVk1eIJuRwxRlzXhAVABlXyfR7YtQtPvvY69Pf3IEbqilAuM7ctxRvEiJl+seGcbMoCcvkevQ+jafZjLZUX7XqOEy4cgv42ndIzsKOez8H0RzmwXA0trNXPg89++q3RyrGNuOmzdzrfR3/LJNvRJ1203GUvm18kTCmCNR+4HeGarSN45e9eh+n5Rey84GL09BSkuWQXWMe3Q5/ESYJQFVY+mO9qEZ1ZNoqN0VI98OAF2rEArhvOymce9DDR+iDLVSgFyxka/uu0WPO33cJIVyu7Mzm6m4ob3MqiipZjpNo09C7iTjnI1IQc4aFHHsEll12CYk8OYdsmDSTYMachJhX5xXS+X+lWPMloO41Eml2CeQSxtJiSdfKp60blkfAcKZ19VxSuOurn53TNbC7b6WAIkJBVDD79yZuilSOj+JcfH8b+o1OOUEY6nMN+HfWl44OiLuDgUxsKuyfewEff8hJkyE5oA+efv1PmaHp6EhW2SDrY0IQXF7NfuZjgSRLJu0ERTY/HcLm4HaE6bbSo27Dt3xQM2e51uKvSHUt7lrthM8nn8qH5M2o6SW3Gi3Ik92W/6Neh44NdP5SEx+qXBq808OADj+CKyy9DLFFH1JxzFFgyOvjeS5ibn8fA0EoUewaEUadSBSRTecRTRcRSBfnSSm1JG1wIlY8lVBa1+/gon03Y0mhOLlDKQ7NdQ/D5z70zIuXl8FwM/377Y6R3uZTIqkTRstFBZlrONW9cZJbp4mETH33D72B4YBBnzkxgw/qN2LRpE0qlBQmY1RXeuCNcNmcR0uPEGxcJ+MiQloDXtADFlfccAKENtazk5zXVm2TTeAZORvnUu8rCWITr5cTr/Obo2qJa5t1+dIPPqb0W2zo46qxD12wTMipuo9lu4r57H8Q1V12LIFlBo3bWmrXVPWHMSUGeehNG43FNCygUhxBPFhBPMl0qIEiYf2dNmPez7MNiIlvLlqwsr804xXfZczALQY/g37/0/ujs3CzGV63DOz/9E7TcOB5vetgC6X2wvrvkSsV7jwjwScM2bn7VM7BufFTBwd49B3HJJZdg3bp1OHv2LCqEwxRtW5hOXy0hsP5Jv9JiVSQ8h2clLNsX9OmLqR1us6mcKAjLl/RcbuzYCl7YRrfxjEbTVm9efUTu677dAMl+WxGsS4WWa+xy889r+MKHWJ3uHe+9935cffU1GFkxALYU+xFGwuSdK1P3tCPw6ZqKC9JoRSlEEQnrxI2bypO5FuZiDIvwpHTen8UICj7O4SexlDZLgsHfd7/+kWj/6ZMYHx7Cl247jj1Hpzo+RSaPzdNy1o4d6Adtiepq5W29ICI8+9L1+L1nXSU2JO3+3r17cemllwpvJetvZnbaWYWYmrhVrXILQuYGw35uGFVGXC7p0yL+nL64Q3xz+aUJxAoRhpEvazuJjDaz3K96VqWn9DhP3YnFfKDli8ACGahZywaQLA+0+BIiIzgivQdG7rnnXjz1addjbOUYYlma94TGIPFZWxr3tIyG6+g9aRYKckXkC3kkUnnX+xTDQmkRZ86excLCrFnTtuWz8vl6P3N1JKtnM0ytYmZxv/f1D0YnpubUpHx6MYav/ehxPagvjWnhPEOQQibfN0qiFYRIJNOKfjX3ImyhEKvjIze9VNUh0kwYeT7y8KM4//zzsXnzZj3AwUN75Zv4YNJcji1wmqvyVaMu4dIcaTe6tgnrPjSWoQffmdQnU0YIp0bL50i4XW31qYw3rWbGfYDXbaE516w7uolDn8gu8ZbMPud4Zq5G2+IG9dYhAirVCu655x5c/4ynY+eFF2oQC5+vk3WcswmNC95xL9JkC9iWuwO/QalIM3OzapEpl22kBFVM1lANdsSWyfJIIPjfr70/ml+q4tTsPDasWYc3ffqOjnCNrWipAp9MjVFZYPOaAezcsQPbz9uAWz75H1gx2ovX/P7TkE3FUC7VZFrT6ZzmRTDUZ68pWxN37NiBQjGHAwf2yzQp8SY3yY01oKkV66/eEGtQezJsKyDz8B9pKIcPHcGhQ0dw9NgxlduuuupKrF09rqCF+Cs3j0YykLSuQIqL1aURWTDmYE43XW65cDtq7KJvXudcAXd5VsKFljEm+S58h1/96le44ZnPUBEhzplQ2nHehzyxJt0dIGZ+ffmzuu3kGKl87tLiPM6emcRcqaJqELsiFFxpqk0K2Tznb1G4X3l31IxiOHDiDMZWDOPLtx7AniNTUutUMsC60V485bpLce1F5yMb53xHmkBruWADcTqbkuuYmJoS7tlb6EVPoYBUOq2RCIlkVkA3AXXWQM/bvk0shwP796LJAWGctUEwQw3EVs/MZmwWpK9fcrFKSwtaIHKEjp84gX37DuKO2+5ET28fLr1kJ+LtJlauHsOmzZu0qTRPg01W7BdS7mrm2gvZAjuL/I1GYwv6xC+vUfx3n5J4rVoeYBkUa0Ej3+PBB3bhhhuejiuuvdoVZbqdeL92k2UQqv2bFS4sVXQBbKuJ2akzmJ6ZVFGgEcVRbxmGvLRUsljFtdzmC33a5MF3vvLuiJPfjs/MKj87ORvDV3/0ILLxGN78it/CRTs2qfdn4uRprN6wRfRLmuC9j+9SJ3krTOKXd/1CZcCFxUUc2HsAr3jZy9WZRhPBIWJkOxBmSybi2LN3H87btk1Fht27H9XIAj7sxJmzqoyQj0VWA3egLb7xsirVJWkE2zsOHTqMYydPYW1xCFG9qsbpRrWKRgJYt20ThoaHUGs1JVzyi/ni3Nm+/so/GwpmVBV/Dx+FPlHIHo6k2yBa1HVb54rJR8vVag27HnwIT3/GM3HFNU8WPCg2yzJi4BOjfH8lu7frxgBQa9QxffoYSgtzaJBRGhJnCCXcKGa57fzcrA2CITrXDFHs7bcJct/60s3UZsyXazg9s4Btm7bgE1/5MV7wjCuRj1XVS1ro68emHRcjiidRr8yhVpoWmlKuR8jn+9yIO0dRbbUxPz2jZyXXltrLB2ZZjLSRXKGA++67X1E02RuPPvIgFifP4rvf+g4ufdKVWDE2rs/5sN4HKqwPc3RRvdHC8ePHcWTfQQynsujLs8WSvUllzC8tYmjtKM7fsVUWZrFcFR87xdGDyVQnhbCufqONdiNkC+TSKeK+TzSLnrZjsQjZKOf6w27RgRpM4T70yMN4+tOegSuvuVp14N9kFcx3L0fNmO/bZCFq4/SZ48qJbaRSiKpGB4bIZQoIE1nUHHGuUq6hXCnLlTFmoUtU0/c3v/guX0XE3hOTippXbdyJ3Y89gFw8wujYWvSu3IAUZz9FTTTrC2jXltAKEsgWBhUFSqOoOfU6ij19aNXqWJif10JQo7lgyuViceSKBfT19eKB+x7EwNAgxkZHcdu3vykh1dshRtas0kPy4WzhLX1imjE7O4elSgUTExM4su8A+pFCf46d7m1U6lX1xuYGcrjimisUMbZiccwvllEikzDmmIjkHblZEn4DeXYjsWP6MFZ+yDI0k06/7SBS189kJUDmmDZNx3OmVbsNgHK5ir379uGaq6/FVddd64r8Li53LS+/JmyxUuqYmT2Lec7LrNfdcE9oXbnxyK9WR2Isg6Umo27bGKTzkG7D9hXSbRinKCf+1hf+2nqFogBHpmYRhgEuu+wq1JpttOp1TUDjWFo+dbO6iKWFKeVjAyMczROhNDeD5vw82tk8hsZXCW2pl5aEexriExPgnsykBZnx79TM3t4B7Nr1oBj7e++/D5kgwoatm9FkWp+yGipRGmbTjKa5mATTZ+fnMTM9g8P7D2FxehYjff3oydA8BSgOD6IwOoih0eEun1Usw4baNX0hnNxhBmikqXLhatWqgjHOgBalpc58NYZiT9GE6xA0HzF7zhN98HJTbmkKp93VsHv3HlzzlKfgmmuu6RT5zQqFnTHBNJmMNRrVRUyeOY7y4oKCI2IJFKZvDyE8KUvBHJbfEynML9VYFHWBeyDOMiFhC+hamJqcRPDtL1qXH83JbLmOU9OLuJBR7dAqzaZi7hnGDRWZO3tMTcbJbEFQcCpJQhwDoQYKhX65FvaJEvGamZhyILojgGWMrUeB0c/1cvBzJot779+FdatWYf8v70Ihn8OazRsxx0Atk1IVBCmaTtMG+v75xUVUyuxqT8tKsH9GMKLLc1nFYpuG9e3GbEYTgXe1lqq0ro/ST1szN2dUEu+mWSaQ0hQ6VVqYFz5r44KNxiK+kpvURgEzNqAZNBpOt1uBdd9HH3sc1z31qXjyk+lzO0Qv+Uj+ndy0ytIcJk+fQLW6KH53k0WSJsn7ZFOSvmpIFAsMCt5iFmSSgltpkhBhJVdqqjjXgcGP5FiJ2fHNf7FGMI3yDAPsPTmJbVs3o39oFaIgjvrCAtJ9vRJYPGgJzFAaodJgVlFoNmM7nNQaLiyF3Wq0MDs13WFAk1wm8jY1OMEZy2lpMCm19/7qAawZHMCpvXsxso4T2xqkIyKWylgwwiqHgxUJnfgitpkkTmo1890FLLoN5FxMgyO7RQXLGQ0dEuOSlB5XeaFWW2pjuTsjeRLqOW5vbm5GP+dQElJX89mcKjJiNTLPThqZrlKrYvfj+3DtU67F1ddcw+FMDg82hGx+ZgIzE2fUokJNVn8PzXAUiO9MFsw5QnUTbLVF4glUqk2A9CNCrK226Lj9w6PdGdWsBbNyRuGqYC06TIADpyawdv1GbNywFW2mEEQWHZZKDWCnm3BZ9qLG0+jt7Te/26yhVisjrDVEDR0eXYG9j+8RLKnPtw37ZARLn8bFKHJCTC6L0mIZpycmUDl6DGs2rsfi4oxeIl3oRZDKoCnGhJ/h6HqZPA7qWCEUrwB117qpblyVYq3tXjveIQF8Ht8uaiOZ3Owt109rBQWrSrEUqTmTRJTccOuwXcfc7AxmZ6fR19urLkc/zY4bmJp7+PAxXHX1VRJuFBi3eebsMXNj6vUx00sqkjfzUAspe+9c2tQBMwwBU9kyHsMPf3gH1m7chPFVaxTcNVshCn0DHfoOPyn//81/eWvEtMBrxHypghMzJTz7Wb+l7jWNi3YDNTybkeY4mUkinbIxAkxVGs0qmuUS2osV9K/fpAapvbv3iF7jUweLmq13lSMDucv7+wf1/Z7778O6sTUIykvYs/8hjK7bjFTvoCoivvLj5CRhCfJ04wo0Es+xHXwBX9MAHCfYpx0eyvTVFJ9HL09tuqU7K+WpLqwWDb+pBIFIo3lfrs3kmTMcsY5igZkB90MME5MTuPa6a7Bz5zZMnT2OWpl9s37crnG2WdNlPup7fzS7QGbVI2dPqC3HOA8jwkf/5uNIpnO45tqnYMt55yMv1wRkclmHt9scseC/PvfmSFV8B6k1WxHueugx/P4LXyK+LbvD+SCznP+QTGP16rXadQl1dzNftKJ1q15FbWZGbSljm7YreGLktm/Po520wUAEQ1E4foeLTIQpl88p79z92B70sojdm1c+J0L8slKar7VbwYBgipkl0VAcFUXENd/muWyEjwf4fa7pUyDTYqsYqStedVOruxpIYa0kFnTan+05bF4yf07OFznHQdhW8/PExBnFB9c/5ToU8zarmo/ZaFpXQE4IkrV0dm7C6MW5ZlpF8+OOrOhBjlgMJ06ewQc/+BHNCxsaWYHXv+ktij0azRB5Np4x3FCfcYTgP/7xzXpUmlz+WIXmvYewfst2jPT348DBw9KQy654skwQc82+oRUqDRqDnuMLaoimZxGL2siOb0CChyjEjPz16MMPqNWh07SdMNCbIb1FxAl1l7MT7pe/vAcbNm1SSO99pC/h+QqO95Uap6eeHYvkrRuCwZu1cHQrPsYi8f/7EqJPRfzPbbJbl9WhAMmPTHQjkjT5TZzh7qR0r/26ju8NFvegjVw6iXy2hWaNuWoLmYwbdURzy1JdJ8c1IXeY252GvHNRM6aTd/70LvzdJz8j4W2/4EK84+b3qomP8Gg2Y/mtbcoAwb9/5k1OuJaYs8Q2PbeAh/YcwqXbt2KhHql01T+4Ev/38+9jxchKjK0/D/EgrcixVZvH0vxZpEoNpIdWozC21pj5Lig4cng/pqcmdIKIaY2ZU/lfzk526BXH+iwuLOHw8eMYGVnhGJR2/IpnGcp8uglxHYTHjTDwJns5mc5rpc8GTE3cizu1tAmxbn8otiABzj2rousuDuz9szYGBehmdvjZVJ4HaSXFNtKZvEYg9fcNo16dRKs+a5Qj+/WOpvp5HF04wz/nE8CUII6//btP466771d6+Ozn/jb+5BWvVOBrU+2t48BKnKBw36gJcmEH/LaW/Xt2H8TGNWtw4YWXotA3iPnZWey672dYsXIMW3dchky6iPLCBA7tuw+57ADG+sfRt+UicXqtucpSAx7S8OB9dyNOrpDj+fA7fa6OmnE9OkX2GQUBfvqzu3DxZZcr9fGC8EwMn6f6n1sB3gKp5ZrZiYZdXqmKjINqrH5qYvAm2goMFlVbIOX1yBMTltNeu/hzJwZww0qNueEHkLLQQmw7jkwuj6HBQZTrVcSjEpq1WZc7n0vG0939XI/fUECgaX/t629CtUpX2MZ1T3s6Xvryl+tMKP5erdFQFuKnCwVf/4c36LUpXJksle9CHDo1hU1bz8PI8CjSuQJ6BwaRipPUFaFaW8TxA48gm4ihf8UmJHODqv4Ucz0a7mE5HxecM/qr2PXAPZrA5isXFlg588yyXTyOniJpJik8sOsRDA6v6IzD96R240tZ0dvCYMe2kCl29BbHenyif9VMLKe1DF7oIkQJdYgTQxjXwNQpF1rlyIRtDeF2gXPcgxMGzbVr7O0Ef4qAk7bQyQzbSQrKQ+MRjwaYVm7rvzoQaOcnnlprEb+n+0zNzOFTn/4X9PYNYnJiApu2bcefvOzlnQYCOlaS61QPZo78b59+gzTXgoouC35msYTN2y9BNstjYQjAk4zdxOLcWcTQQKFvDPneFeDZBlxTTVlJsaXQIDkLQCKcOrIfU8zp2k5THAfI+1vOgOTn8wVrS6xVG3hs736sWrOu033gCWjLYFg3YceqPN6P+vfgGikgcX6QG8RXfTRYzD2fX0uNmu+0itiIJPP1ftxg12BaccB3OnY7Eq3ebFCppwslk2zKTulUFn6nzw0Zn4RltBqz2lBesB1b4SpTy+FJXwI8PTmDNjJsA1Ne/Nhjj+OGZz5LWY02nhusQsurkunXPvlaPbknZ1NDWACu1ptYt+V8FPuGNMm8Xivj7v/7KebnprB9xw6s2bgdxYFx8AXIv+WD0wd73JYPVy4tYveuX6G3bwBziyRac8QdI1L7zuCHs5Ysz7N+VP7stjt+hksuvVz5ogEmHIVnpsenQNREnYe0bFyNN2kqCngSmaOqGnRIgfvJriZwC4is8/CJvUjeWpwjANfD5FOmznBxZ04NX7aUT2iczjmyYCuTIaLXRNRaQipJFkV3/qWE60bwWKuSoWxyQSywRhGmSzWEETtCjMZaXqwglc1i1ao1+igbC7zbYQQf/OunXhdxp1pfj43jY1sDnXMdCWy74CIdWrF/zx7cdtvt2LJpAzZv2Y7x1ZvRjJoYGlmP/oERaS3RJg/FtRs1nDhyEHMzUxgYGMDk3LwwU+/fDNExAUu46YSbeprC3j37EMVS6OnjSPjuCKLlEa4/tMo3mynYcoGQpsI5cr1+rsFgJkjfpqmBmD6lUm65nBbbnWul1EqtIxSEoUky1Y7Evly4SgndsTH2nkYYYFrHAaHV8gKymRgyWY45CgVuLP9yLJyuuV5mqjgOa7Yc6nAsmvtENo0ETyqq19VHzOmwtKJ+I8p6fvXvX6ujZwhONzTyrqkEee22y1HsH9ZBi4sLUzhw4BASyTx2XHAZKrUKZqYmEdaX0De0GgNDo+rGsxEANpCkPDelUbezCwvIZbKYWeBQLMsLVUiW3zPGhE61omnO51UDZhPxPffuwvYLLrBTTRy8aICT29HkR4mw5ykxNtRSfCcHPviN5lsdfRTsN4EKG+56Ppiy/lc3DYccY47Xd5+z+c/eLHd51f6kFPEEHZxoRRMOBW8hk0pgeuYsVo+tIOtUmyOZYAdl97wGmXpvO57Qt8QNxEHeUaoPuUI/0qkcEnSV7pwhsJ+ak+fTPPTSql7S+K/+/euiVK4Ho2u3KXlv1BoYWbVeH6Z5TjimXRBY/sQXnJqeQF9vj5sbxY50G7ZlN2P1qISl+VljPnC2w/QCSP46PTOtx+8K1ygx2hQOsert6ZWQ7rjz59h63g4EIqgzv+yO75NwHEvTFtGzLLpzlj1DUGxBD+xbmN0BQCzNcXO2XAqkpfd/duCGKLK+q93P+hAzk2OJSBcyDjWtnQnXNkQ2lRQxsJBLgu+lwMsockilz+2UWB6pL8/teb25uQUcPnwYq9adh7G1W9DTO4hUiiwXg3EJW9qGtf4romd61S9/4vXRiq3nI5HIK6pjlUWtIJW6RgDoFCoOvmzzcKM6cmK22/ANegMCGfQt9L0UFAvNlblpla6IYvEomaDOMCCOx44eQIXXJIHakb6lvQIzLPft6SmqsH7sxGmcmZjCqjVrXM+SI2LTZzsSmZliq/6YkE1QVvN0vKkO2c/G/fnPLE85OhagMyfKLCPHMYlD7doXdLiWEz43P9+Ri0/r4sceklXCAxg5PJtnKK1YOdIZgeSjbzbHxROOmit34BvNXYDGokWbaFcZp06dVA+xmr2jAPFMP1as3YxVqzfrTCYxQlkN0sxmP3nWGgqC7/zrR6P88LhmHBWLPXpQcp3YakiTxLlH3tyaBbNo0s8O5qg6aq2GY8USaCzOqTrk5xSngyRSnEIXAQvVJew9cUQVH5XmNPfBqikKrkjNyWdVCmRN8ud3/QqXX36lDfrQZFULMCgMzy+y/NaFHX4iTydyda353YpbR2spKA83MvjwFsBCWD/Px/hixDYJj7IU6IeNWiBGoRL8NyYnW2OqpQVNERgfHztnWo+iWXfWHwVrYyP8gBd7Tn8e4NJiCSdOntS16ars7Swby6TtfNx4pg/9I+vFN89wyLdC/nPhyuC2H/5bRJw3X2Q3WoizZycdMTzUEGkS1bgIFCJ3K2uNLH+RVuqHTZNpQQ1tc+T8XT/HtvO2I5ctIMuNQVPhpqtz3+86sBstapejslg1xa7v76MwPhbHXb+6T1h2b1+/sxTdoZ8e7vNsCUOa7HwDLrQCGuOSdhbHarx+qUw7O2cYOX+uxm9+TtGNMSRtWJEtMDcCzV5VZyOQ0mr3mmU5sF2XXzW2KIsOXRjUT+JRj0HSpp53K1Lmq0mtOXDwEKpLSxgdXWHjiJQlmCZbI1gSuQIPrqJZziEK0ugdWo+RFStRKPa5Ax/dO99++39ExIz5oJzq3d87pAiMtJZCgR+2vJXaLJSHuRTYzkg+1ZL4SQqE0hkc3bcb85OTWLNmHYYHR5F0A6+lFS4GPDZ1BmfmZ7UA1Fz+G30wtZ8Cpu/VOKBEHNPT8zh27BS2nbdD7kEpjitg+2jZzLAhQ/7L/0zYhIMrO4L0vUeuK74DUWpD2KQ4/ucn1Sr/V5Rscyq8gHk93pe12XJ5Tr2ymTQ7BZYNanEdi517KNWhW3LDXpbVco8cOaLDL0aGhxXrEG+3KnW3GuWRmGQmh0K+1wWjVvM+OzGHgRWrse2Cy9HX02co4T2/+l5EVsKx4ydQKPbI52peAzHfXI9elCdv0Lf2FHskTHZ385i3hblppNI5jI4MY/L4KTS444YG1aeSQEJlMl/p8AhRI2rhwf2PK1ezaNbGDXCHCs1JsVJUEIxG6PaXd92LKy6/Si/g/amZZwcj+omrHXDZRu8qFVgGxnt4UubRFRYsJ7Q0iD/r/N2fgOb8qyJmFzCRQcFrzc3PLru/ggAAIABJREFUYKk0i9Xjo3pW+XBtnG5HIwkOZmq5Zaj9LQRxOwyTm4Zs0aNHj2J2ZkbnFRFZ0nFvbnC5z7t9KuZNN3nQFC6j41SSGsw4xI7RmZgtYdsFV2H9xi0IfvqT/4h2P/4YVq9ZqzPouHttJA7HyfbKB/OXaNd1OKBjYnBw1uzUpDjIuUQKpYkZDA0MdNAfP9p3OQBgfqeFr3//O9i0eaOrYNh4Wz6cZzIwnCfbga2Kjzy6B4MDI+jrH3Qmx+G3rLE602vAvfPFjvzmBetrt7YhDFnSoBPXKurJ6SYEX9pz5xe6M+j5b/bsbSzOTmJubgLjq8ZEC1oe2Yp7tOyod4tPLCibmp3DihUFHUXOya/Hjh/DwUOHMTo6it6eHm0e0op8XOHxdD4r51hpgqxGRXEgNZmkRTueNmEnsBlebyOUJmdmECSyCL7++fdEHMG+cs1mjK1ar74Ucl4505+NQuyx1bBsjTHi/EM3PbxeweLsDFYMj6AnkbETpt285nO8moWXyhxFYYkFeO5LX4Z3vuMt6hAXwZ3+F5YSMWKmBvf0FvSgPOzwyJET2on0611UyU9a92mQm2LufKefq7F8croN2zZ15p/5ngySRFZwzVZ+cdWzpAOTQ7WlUlNLi9NYOTqCQj5j2u46EK3Ga5vDa7BVswxF++4P78Dddz+Aj9zyOkxNT2Lf3r2yTr19Zlo5gI2j68lKoYA6DXbuXbhuXTDHxiczFmJgxX5epaFq37QAlUohyPLv/vpFUakWYfV5F2nsnI4hjccwSE4ObGIKaZP0cfTL6vHhGLp2iKF+JtRpHUWz3Ox1nB8fjprSbopDnMrnRNt53p++Gju2b8Hzf/vpehBjRdqsJ0bMFHCxyK4FnuUTx91334ftO3fKBFmC3q3MWGoDQZ8dGo0QKhOgNprzu8p53XytLhZsAZHH1el+6JYYNHHYWK26iNL8FFauHBFA0PGp6jrstDwaNKoGLyIZEVpBGydOz+KTn/o8FkuLGBwYwkteeI1mJtON6Zxg8q3ZoxwDFubmbDgoWzTl9hwJwQWI84x5AlaasupgoExIdWUNlyenKOMQS9LOHpZb+shNvxedd+l16B8dw749+3QE2tEjR7CwsISt23dgYHBYlYZimvMu8hjs6UdagRIRlq4YrRtx2Q98+N6o4czJExhZOYZ4Oid/84I/fx0WZkt44xtfgeFBzoOgcM0kUWv5kplMSvejPz5y+DjiqSyGh0dd173ddzlAYSaXARePYHU1WH8MuSvvdQKbTnXHepE8ZCgNceNwORvq7JkTWDHSp/NwOTGGhAav4b6Wa6ObzBw3eARAixScCN+97Q5841s/VEtlNhPH8OAw3vTGF4v1SQ3XmcANbiIDQrRpHN+M0/uMPGBf/Deef3Tq9Gk0iRnks4J0h0ZGFQel06a9VBSRIFyeH3zz6x+Phletx5mTp7Rc2XQSX/rCl7B27Tpceunl4JTwzRu2okedA8ZW+E1fFK49ibwTKxGoLc3h5z+9E2s2bMV2jjCKqHUhXvyXb8HZ09PI5GL467e8FmmejcuxO9JAlsmskM+UiFaEk7+PHD2B0RVjRrBLpmXyvLXwEKKHNm1mRld7LfvpTqDx5pM/JqfZLFJT7S6sM09NntZpoiOjgx1GiAnVEDrvW71p5jtxk9Q4aysWx/ETp/GuD34KYcsg1mw6hcGBAXz4Q28UT1rAB88jKFn/kxq5NW7fToBRy8oyUEb+lmPzS0uYmyXt1w6SLvb2iJyXz/WKd002i1lAd8T5F//pAxFz1rNnp3HFFZfjJ7ffpl1D9kUmSElT1W3vGAkdGTrfpS53tWCylbOFiCzIyhKWJk/j9NFDaCbyuPpZv+PGGNghha9427vEDuRqXbhzM17yB7+tUXsEJhhUkBhO08ygyqbJJoQ1U3PZq6Qh1X4QqZu/yMdRpcnNjrDJag5udCiQByCkqRylELfpdqwgcbdPT51BPN7G+PhKd0aPHVbh0yLvV7WHdZybzV8mIcGDIAxA9+zbh4//w9dVClXuzkOVB3rxzre/WvEF72/zH+3EFJpQ+uaFuRlZBp2P64oZPuQ3q8gzI1qoN9nGkxfgo9abZEbvzkEognY9h+pD73ldxItf9aQn48CBA3rZiy6+GKkwQDHtiFwqR51rdulfNAa2ZsemVOenEOdIQJ5Z16jLvMdSeay96MmaYkoHL78UAH9+8y3YvXevMzltvOwPfxc7tm+ynNoFVSSAc3cyyODP9x88ikQiJy1jBYQ/Y4DV8bXLqkIetfKEuu6UmbYKI57KqxJlLMDszIRGGaxeNSZBG4fbGqS9ufeaK+qsw5c5Q5pDxJSJRhGOnziFvr5+ZAsFvOEtH0bDzY1MpjMY7C1IuFQO46W7yTgc6En6Ljdcg90PFU0/50ZkWUE+mNNuOJRb5/4lELYthdTQz5z1QdGi8GgaNb3FHI/q5re+Mrr++qcaOH3oMK580lVAM8Rwpsd6PL05O2d0fQvVyrxYfj++7Xb86r4HdajgZZs3Yf3YKMbGV6NnYBgD4+vVKW6zRzwJLMBfffQTuPu++115ylzBe972F+DBO9Q8Etf5kNydjCopyPnFEg4dOq42FC484U5G8fQ1Hic2SNATD2yulI+W+TtqHWGJLGOp1vzcpGYhr141LsjTJqC7QybF+DB/p5O3NbbQzCZhR54qcmDfbhQKWUxOTaspfOXqNVi7lodo5fD/Xvse1Oo8M5gDv1IY6CniHW97tdW7SSrUSAbLsdVsLetBrW6qTKp7xY2KlMkYed9X3hIJ6170AJOdY2A5tT8mT3L78Xe/IFL6bbf9RCnBti3bcPXOy5COudFzHkxXrYrMvxDlyhz27XscP/jBDzAzXxadc7C3B5tWrcUN19+AdTyQKZ0hhKMN0nHF+kMM7//MZ/Djn/+iU3ukW/jWFz+FBx9/VIINknEtNmugFC5NGVtIbrvtDlz15GtQrzfRFJhgG8YPlubOJiZtrBIrpxH35eBuCqdY6FHhY7E0i3q9jFWrVmgD+aGhDGgsv7RyngTrThmza1LrQ0xNnsHBgwcE7Oi6xaJKlWxyY/F8aHAUr3/jLSpdKv/MJtCX78Et7329jRkkDVjHxbj8OYwUS6jGnUions4vK4l2Oxk4zoj/7kcUel61jjBQTGD15g6n7Nv/+Q/R3Xfdjf6BQfnNi7ftxNjgCOKcsuL6beT0XWms0Szj8d0P4Xvf/S4K2SzGCj3YsmYtVq5YgZ7R1cgODKnMJ5RIp2B2kSJFlhHwsS98Cd/58e1d4SaTeOlzrsOhk8dxw7OeocCAmknmIBeOU8wZVd7/wC4MD41oLmVPbz8WFlxwoSZrM/sMjLjgZI/QtHlghCjc7NykArqxsRXoLRbttBGnmZ1ZG44kJ3qs01g7l7aF+QWOK2AbiE2Y9XwqahGJgTxmhlaBh1fc8uHPolSy7ox4OoHefAEfeP+bHCfKprZy6IufocwgkZuYm4Gon01BT1rLS2RTcLopoyfuGY3SY+reNnYO+Xr7G/8oklNmJ3wqhUu3XYw0eUY698ZOu1RJzCrlKJWmceet38OK3iKGyK+KJ5RM50fHke4ftqiXeVbMGr40CoXDOhs1tBo1LC0s4HP/+S388N77O0E3g4DBZF0R37btW/GU66/XHAn6E1I1RS5rRzh2/DiGh0YxNzePM2cnMDQ8iv6BAWkTy5OitOjYPU55M1YJBUJh9/X1YGRkQEL36UU3Z3Ujf6Wty879pSYT0C8tSqhVtsu4Ide8htGDUvJ1misZBHbWXzqFv//M13HmtKtpp5LozWfxznf8hW3WJEuCPEHMiPCcqZFMZJ2JhgrxBubknZ9lA3oDrbpNjvUzvbS2oiF1fbhtBnfMzYfefaPMcjFfQD6VwQUbtik2NkoKDzG04dKRQP4Qs4f3I5ydFVmOF8rlCyiOrES6f9TNfnD0Fe52oj/Vsk6VRtOO29514BC+8oPbcHi2y/7jgl+ycdgCmaiN887fgU3beE57XmXInl4Ook5ganJaXQ/ciHzJqalpzMzM2GCUmLV9avcHQD6fRX9/HwY0G9HoJ5aFdyfOdRAmP16XTAs3B5LPWqtUceb0aUycPSNTyCNiOHhT4xjIKNE0dNa5Gzp6hpG82kUTSfz7//wEj+8+pHuyJbUnn8Z7b/5LG0TmFl9pUo6QL/0nD/AwJicFqQntqZy7r9F1WjxeQH27bhiqywhkWT17Q5mBnRYevO/tr1J/biqRwtjwCmxYMY6kWh9ddOxaDgk/EviefvwRxJT2hEjnC+ihYIvWDKZ2SB5VzinfHhliEzNbT7jAQUxpwnd/9gvcdvc9jh8M5bTPvup8ZIhO5bJIF9g914vBoWH09PYqOhYzslbD9PQsBgYNwxYJzc2y8JwmY9z70UW+qmLRvszW8vmVLne1uVA0s+zlYcddC/OzU2r24pxGf+gGy3xceG4KBn40wfSBQvCWEdp41t6P7rwXP/v5A2aWkwkJ9z3vfIMazwmQWDRuw0KTaeatHE+UNgKgH3LKe+j4c0Ph7OBIHqdacfSiLljj82KRBv1RfR96141KhRixDff2YcPoSvDgTD/7USmQO4I7rNdQOrIfsXaAdC6LXG8f4qkcqqUyyiwibNqKVLFXJ2VxxAJrssKklUr5CkwM//vTO/Hxz3zWem9IR8lk8OG3vhbzC3PI9RQwV1rQGQMUDflXg6PD8r90EzPTs3ZatNpRLD9VoVo5rZHh/J996VY7ezlo6e6r6pAOQbSSHjfP92+9A0vlBjZvXofVYyPq89H0VJ1cUhELhc+txvCwpT5aXlusRzeXmQDLfQ/twbe/+38WGNEsFzJ4+03/D6OjIxKgprRyPiOggxfTghHJ3aYw7Xp2wkuXdO+Zm3Zws6FcPl2jxVJly5Jwe99//ui7Ipaa+vv6keFAj/ISkjFrsvJAAf+cyqYRcpTf5FmwNsTLNGtEayw6K46tQW583AZcqZ+UQmXJ71xIkuz42+69F7d89GMd4TItufWrX9JAMz4UB3sQ0OfDz8xPo9pq6HAMCXeGDWkplxYYHu2jQ76XMRJMRa1Y77TXUWU8AMEDl6xxmTQZ5qsVAQnTM/M4dPQ09u09iMNHTugouysuvgAjwwVEnODGsZWMSLlWzWVn5zqYUGa11cLEdAmf/cL/mHCSCfQWsvjL171MgSfdjabPuCNTWxGU65L7zdydqRIHenpivEb2u5KnL5xo5kUQE3GCmiyNV9sUG7vdCTAP/PC/VbYm84C788zxowjanGtkfKMkT3TmYLFiBgEhsH37NYIg29OPAgvy2YKqFOzPpTnQ+RmJlHYjMWJiwjaBjlvJ2kzuevRxvP2975EuUXPZp3vrv35ZwtWp0hSSK5izk+705FnUgppaFOdm5+0AYo2nd+Q68bGMmd8Vbidec4rsit6aS9wWskQhsFG80axbLh4Ztm2RsJHeHn1sL35170NYLFVw3bVX4rxNq9FoVux+jgnpo+YOzTaIYanWwic+9a+6N013sZDBm9/4p2qmozknNswhbUaZpY5EYL+UqkIqX5pSdI4RaDQ7tCC5pERcRRu6iqXFBVeL9sfgucHhu370DVdM4WG7IWYnT2FhelJmWQm4qxVm+iy4qR0/pVn6if4RJHM9iCcNKGjWKhrn/uiDD+PA0WMyw8PDI1gxvhIjwyPqITWzk8VDB4/gbe99X6crgWfhfP9rX9FRLOcOs7YF5gY4NnkcyQyHrlggxdTBBool3elY3U6+31ihcucjUbCLiyXc8dNf4KKLLhAQohRe+C7BBJdQaBNwTqTVoE+emsTP7noQp06dwW8983qMjfYhbHAarSv+O/qrzt9jp3wb+JtPfEWCIlqXy6fx1je/2s7LFeskrRo1kThNWFW66ccb2sRYG75oftUPIVWg5F2SG0ExO22nf9J9+HhDbuKhH34jErLRamrcT2l2GmdPn9KL6awb1gqpwfksRsm7ZW9uIo1UlqiJTUZjvrhQmsfeA/tw4OBBlMo8ocqalajRzFGf/zvPx9133418Oof5ehvfuO3/rBICoLeniG9+7jPKB0VJRQxN0UaJEkWYnJ3Fl//7G9iyYTWuv+7JOvy3vFTFUmXJdjurIW4soLkTP1/ZxceCDEMslJZw+0/+Dz/40e06COrmm2/C6AiLAw6Zct37SuEYNWsGpdV0ucxkbB4/eRbf++FPlSX83vOejtrStANM/AmWjC/4/CE+8rdfs7pxPKHo/S1/+SrN3+L16FsJK1KDqcmqTrkZV5y6ahuUczq6p7r4oeAUIYNQz29bmJsVE9NvBApa1uSOf/vniNjw5NQZEc0pKpWjWk1MT8+glwXhdFoQ3aq1a9Db36cqBPFMxp8cgsVZEfsOH8QcB4ER3mPUF0SqWTLFYpf5eVu26gUe37MHpycXcOud93XsJs/Cec3znore/n7DZtMplGsGUByarOAb370Vz3zKNXjx7zzXqDl0GfGEpsZMzU9jqcJ5w562Y2ffSqNaLSwulrHr4d14bPchHD16XJ0Nx06e0Dm1N7/jJoyODihuYFM0F4cUIS4Uf9/A+7aYEF3NsdLfrof34Ps/+in+7BV/gkKKXRqLLmfluQ4xpT/v+5svytwyoi8UcrjpzX+mIwI8zzqZsLH6dDdM4ziIjXMjKXhfs+b29IdaaWwDB6O0TfF0nlDCArNyhcfcdAegqcL08Xe+NuKLLtWXUKtUxHxioLHIc+zicUxMTKJaqWJ+dkbnEuw8fweuuvIqMSNJb91z4ABqYRNDK0e1A8+eOaOTMxiveTNXq9bQbjSVwJdqVUzPMtj4b+uLBVAsZvHSF/2WKjAcA8hRCY1aC/NLdTyy7wiedNFWnDe+SlrEDvYCoT5GlywuZG2ICscZ1oMA81U7vuXHt9+FBx/ajanpeaVNrMyQ5VkoZHD0+FFkkmm87z1vw4rRYWnoxNmzGBoi2Zu5qz/pxNXA3FFtqUxS1STGJxTw9MwsvvSV/8YLXvA7GBnIIQrtfL6Y66h41y3/qEMb1U1RyOJNb3gNNmxYa9Ug1wnJP9MCUmg06by3SIeFvOsbNlNtJWM7AJp+Vm04brYW/S+DQnKlvd+X5v7TJ2+OGCm2G3U0a3VMTU1pRA8Xg0M0ieOSlcegIGgRUYkh4ujceAIDw0NYvX69Ruzk01nhtoxyKVxqlaA0IjhNO8yCmpDv6dGC/91nvqYAhuFTf38eb7jx5dJkWgL+/J4H9mD/gcN4yQufjRTzPV2ngfnFeUWDnDtJjdKZd26A2cCKUYytWaPd/PkvfwMPPbJH4AADOsNkk+jtzePw0UOiztzynrdjZGTIQHoXwPmDMbyfs/GB1ozGhSeIwHzT6rIMxtr44te+iac87WlYt7KAZEDqqmnVX73ro6hVeaJYAvlCBq+78ZU4//xtnWKMvwfNq/lcwgE8yKKtaTl8Lp2z60cbsmhfrXY6++mX/UHKlo41NaLI/G+E4F//5W+iM2dOIxUHlpbKDm4rKaLk8C02QWtXsULk+lmGhodRHBpA30C/hn8xVO/v7bP5vxxTSxDc1Vl9ea1UWhJ6k06S1Rjhbz/9dauBBsDAYBE3vvqP9IJsQ9z1yAE89uhe/NFLni0hMLYQsx6BfDmxXTtjz8bl816Mbgl4CIduhfjvb/0Iv7jrATuwjvQdca+TGB7qx76D+/T7H3zfX2NoaEDvzGfxjEnr1LMFYkSuAr0OnrBeJ8KFJMpzQo8jYeALX/0GnvPcF2B0MEBe/TpJ3PT2DwpfFpO0kMFfvOYVuPCi81T+ZKRO7SI6x89afMFOwIxoNjzPj0Il8sWtJSVxETOb9jzvi9ZSE3S46Vx9mvGFNPcDN98Y2bwKs9fUAiXXjmXPCJoLx7lSqqUOD6Gnj6U2Kw5QW0lUJzDPxaHm0m9RA/1sRZXbGg1NdWVfEa//uS98y005BUZG+vCaV/2hFmrvgVO4554H8cd//LvCYBmpas6FO2SZoRLNvDr53GljFDIDHHUHGDSGn/z8XvzgB3eq61wYsOqmCawaX4FHHntE2POHP/AuHTDJ5zO41SJ/ai8jcT6nHcJkxQhWxGgiqT18H76faqzcdO0YPvyJz+LNr38dBnptI77vQ5/EsaMntSFYGnz1K/8Il19xkfwwn1HMTOWnVr7zG4w1b17bxtvbsTN+SKnaVTIZbfIyzyHmsLNc1obOOKKfSzwRfPDdr43UOeBAc2qg8XTbMq+TUzMYGBjUgQuM0AYHhzoDr7kQWmROdOG0NXcMGqmwxFfn/7+mzgRM8rK6+re6uqqrqvfu6dl7mE0WJUgMuMRoTBRQQRQ3cIsRo3GJC4gmn1E/RFFRZI3osKkMoCCMjiIiYFyeSECIRDZlHJwZnH3tfe+qPL9z3reG+Z58CNNd9f+/y13OPffcoUNKVQApAPt5AP4dJGjd9T+QYjgLM7hiUfzzu8+KTZv/HL/5zRPxutNfprzQxDWzHAWwpwme+By+2/IAqSe1xQstxkKhEPfd/9u47fa7dHP5XTYJtuXa1SvjgQcfEKXmy1/8TPR0eTxq4tMYedJocg6Vv5+GryyHrxl5ibJKGpNzYuz65Mx8XH75dfGBD5wdC/p7Yt01N8Z9v35AaU2t1hbveudZ8Tcveb5UgNzZ4PWzUAva1h6okbsTWR8+H2tnQl/u9ncerkGRiSudiLtpvdy9WLjg39/X0EDf6UmdDnBhnDlmWfaeua7phbghrplOC2Vhk/BVFKr53+TBuV2Dk5h/j5/Hd+PDiaQB4S/72ndihoEOUYg1awfjnW99fTz0v1uj0jYff3X8WlFH8iTKzIIQ7JhoNA4cioosAfABVogqCXT4vcce2xQ33LBBCFmuiZLWHTG4ODY9+Yjwq0998rzo6eqQec+Fb0N/ZjVymCkhqqmNxU96ysJjpIfsrv6MkBErPPjw49FW6Yrjjz8yfnLnvXHLLaBULVFrr8Q73/bG+OsXnxBMBNOBorUkbRALlxvSvNHzMZfmQTCmRj+Hoh0WrJxq5GksEHPpWWPcFxaK59WluPAzH9Bw5PxFRKqCx5IjR7LOI1U8ExZ6J8ER/67xoU11VacfsO91O2emjKBMTMgc47s5GBSpucmXXHmTBxg2GnHssc+ONWtWaibCP7/7zT5YSWoPC8aDq1swUX0wzbIUktKzOaMGwKGRpH69Hk88sTmuumq99LWEtMksl2PlYH8s6m2NcqU9Xvbyl8vc85xiD6r+7HlJLD5Sh/ZzdlVsprHeZwAmuIYMgKh40ojPnH9xvOe974r9+/fFlVdc5c2ttcWZZ74uTjrppWJS8gdzz58sUGIeVkrjQMkSV4t/8t3zFC2ExbeZNy31O2BUfs/jeIgNStLLbETh0i+d1wAmhIEIdaSr3VrHWbCSsJybLXYf5vAZAwSFeWoo43xMT9G62BZtpAtQRPOMHtKooSFNaVbQkPpcr7r61pieqysXpSPulFeeGgt7W6Ov19oYfAZ5MvmsemPnLS9I4CBTmAKgjLGyqdR+M3l781N/josvvloLlAF9grMjlvfF2sGuWLhkWRx1zLGpUTu1qmjitYv+fJf8bMLORe1JbaeqIqnHiWJ6nnflAdMciief2ha1Sk+Mjw/F5z9/kcxytdYWZ5zxqjj9tJNFf82WgvdkkvaSJUv03Xr+BpPGcEOppygBKmTd6kxMbgGzrHJsGgcEmOPyX1IjuPhCFOTmdePUbVcuxdT0lFo4UXbjIQiQ1AgmUwVh2reD06yTnIrk+t+tqLrNij+kemkaboHvYzGA31iQT3/2yphJEzf57y/4y+PjNae+yN+RaK7Mqmvv7IoOdf2B+1YkvYB2IldVFodyJYOqEgmdlIf/9tRT2+KrX71GYpnCdyGYtbXFimX9ceTKnli5eo3+L4MFKNlNTdPF759VOsG/QWZLEom55dPIFT22ZplwgFgnlSgI6orFuPyya+PU014Tnz3/Av03eNinn/qKeN0Zr7EWFwFUElaxT6eEWJMlsb9HhMxUG/7dFbQ8Y8mFHd30dBhFrCikrsCCW1gKXzz/QzLL9huMDavo5sBkR/Hbzj0JRaZyGl/iyMw8JvnmFGXzd5hrlgb+EsOP9flsmMaFFgUXfur8K2Iaud96I1auWhnHH7M2XvLi45TL8jM8A9ZCUgAUtEuOQMXrFVQ6IT+oocDyxZ5BYEGVYuzcuSs+97krgiGWecPowlu2uC9OeO6KWLpsmcRHmd2jZjANIMbMH564hQBJ5imbVWi1ujmIb+IZG2RDnslRr1Ey/Px3bt4Y07P1+MlPfpIsWjle/rK/jre97cwotvo9OA7auLTZYohyaUg99Tm4uYo4aiqpaENTMJUyAzaVOEP7xHgbPYO5z4WvfP4jDaU1QnFKQkkoqzHRS3oUSZ+KDcrSsyTKUF/UvJSCCnGOEueWVIHPdGOSzRzRs0VAZ1SD/dwX18UErSlRiH86+92xuL81OttLIpVxKjGx5Lxq6m7j8JjPjPnVgqTFbE1AP+NWslwB3zd8aDg+89lLAi1L/DJ5rTZ3SV/87QuP0fTKvoEBpWaKUDWVy9MsiSsIpGTmEgPCEkw+YKqhAu8lYZU8clUSi0qQC7F1247Yu288Lr30Uh1wbu7fvPj58c5/fKtKc6r8JI0rgCEdklQRkzVIU8fNscpDJ3NRwyp8afxhsxzoqljOXmaicMVXPi4dKh4Kk4Z/9W21U9ZocfXPOnI0q9AviJkEKeLXOQhssG+xA56sNWX/WU3mzg1hnz7/yhif8dTLcz/60VgyUIxSSyGmZ2d0uPoWLFDNFoyWZ8L/aBpYkj5QHXaGIMcLRUWFQ8PB43uph55/wWUxpRl4vFtZm7t0cW+c8rK/VBMWsgNW4TEYwmJZSTUR0xKZnYzAfcHuJsQW5Ll9OfVyAcXrxQ0kkPvfh/8YV1x5pVwIEe6JJzw33vf+s5s9TWDoziiy9rMtmxl769YiAAAgAElEQVSYMIzd2c8ni76T/i7PtufvFVhWnBK6puvUT5t8xcWfaDQ1m0iIRfWkrdJ0SY9Ys4S8u9Dh3M66gUmO3YGFe1Q9X44/mORnNk7h/JVvIgJdr8f/+/evxJhkaatx7sc+Fov66zF2aEQRMA9Mr7BHx+SgIZ3mCLEf2AwgwGzGKYPhUwFhOO2ga5/57GUxMjbheTutJRVA6P059aQXqNQHFVX12/mkhJP0P9xVN2cWp0iCjhewMnlcTb4hmf2R6bHeABVkY9OmXfHlL18kwIG+4788/i/iQx96jw8An0Wem2YkONhMaquJdapjlEbeSXEoNaxlgdECtfZ02HMc5EawpOJ3+Vc+3uAH3F7JiJh2J84pFUpdI82e1rlZz//Jcgd0mOXc1g9qYjQbxC2m3IcP6ekDngTF8qH55Ke+EuPTpDjtce55H4uB3vmotvLzRsdo3VSvUNaqSowLNpXKCVPH5MPFUSrp1mkRod3A0hwbja9ccm3s2LVPmC3wIyALm/um1/2dwBh8Oe8iYlqLu/sNPXozC/h5xWM2d4IjU5NVdklKmdJomZxJqBbbUognn9wVV1xxhVJHRFD+4thj4rzz/sWxRKksbCHDjskuN62D9iTBouTtKiTI7QG3OkXzaFb7YT+Hg6+MDBa+dsknG8KErT+rBWBjah3tugl6NSoujF+bnpZEDoQwazxk9oNppCoU5IauUkn0zbk6oh0dMTY+IauAuaQQQSQ7OTWris4555wbyxYBt8FaKOgQVGASCsI0cMKLjU9MKHhSb4/gR9tkDY2se7ixfHFibV565bfjT1u3a4PYdN5n4YLueMdbXi1TTy0VtMv8dfqEAe0RyG7IghgBMvtK7kBiZYYpc1McdFyT7ljC1LQtHY1GPPrIlli/fn0cOHAwSuVCHHfss+Occz6oyWp5erZoOVLDoSrErEJH6+wJ79Vea4/hkWFZKxacw0jlCeAIHRO10yQmExbIsQ77NROFyy76RMNyfdYT5ISLPUBLBzcPotbERCxdulTVIk44p2RmZl6mDcFsmabUykGHnqimxaJKhZg+nhiGHxubzcjHzrsgJsanNVv9ox/5aCxfUo35xlyUEuDg0WUEcVYjb6YoSTtSXYVJKkHBXJpcPZfQNIKfb67fGI89sck3F/gRef4F3fGes1+vjc6N3hTuc7Gc71VLCykf35piEaFWSX2dzWdTsxg2SJZoOakYgM+da8zFk3/YGTfddHPs2LEjiq0NlUvPPedfzFcmfxf5kEFPcMYIXl15ymmVpmojuZBaR0VuYG/KdCWMezBUUttR0Jr0qHIWU/j6ZZ9WKgRFRtCVJnUoefUN0Ukg/3XjMTfJ7D8PW8x+QW0ZjUaMT0405W4lRFLEZKYx3o2GAA0i4X/71wtjZMLls5e+9CVx0stfENU2br4DOcBxeMOkShyUant7U5+Sg8rcXfylI3qLhanXVdpRxAzl+O737oyHfvuYbp6Vctqiv7czzv3I25vIDh2DROU51eCgEFRpYljJwtxN0yvV9CS9IMpvinGzFpbaUZK6bKMYjz+xJe677774zf3/rUj7yKPWxKc+9XFN8CKgyyU9tZYkjFhQabmkqhPxBH9wk2Qe5MOyTEWnUHTVcxCym8wUJUGPWLbrrvpcw3bfvlQ9BqkZS2kIeaqQEyfR83OU9KwWBxk7+2YWT62HqdSn/51aI1hwzDURnx6qWo3zPnZ+HBydFEdryZLF8dIXnxgnPu8YpQm69VOUGinFhWitznNJCTw1xGiRBUbYXH5Wf58avjq7uuOHd/4ifvHL+wV8cBg5ML09HfHes18nL2Q6aU0HoUNzAiiEU3EyqzLfXGezFs82rdRxBRSf3HjGQYZ1woFnHZ/asj1+9p//FYODg7Hhe7fpnVatWhH///xPqueIdQMPyGxGdhfLJhkJ6XM5Q2EdXMsGbm1TNgAC5fimoL9jH0zpTUKKKVcvfGvdhRpgwYv5yud2C4fj1EjVR5MMu6IxcM50mngpfEp3b7fMhKBHoLpWN5Kx2ZnZzw3mofiZCy74auzefyjaWsvx3OOeEyef8uroKE1EpcatsXAXQRNRudRcsS5TruNart6fpdIblJtJuvc8/4fn5TnvuudXcc+99zmnlPVpi96e9njXW08RWMPAqqlpUiCrzqFpqVSQyLpWU6TsAoXLb4pyBR7Yt4pOoxTJh0yXWe2Thbj7rl/Ek5v+EC984Qvjqm+s0+KvWb0yPvvZT0dXVy2GhoZlJa0DYkHUGTKAZA2zKAsXi98dGRluSihitbhg7AnW1paUy+bZ9jkYK3zj8s8oHBCzcWpSL81mOGiyVK3TIXJB8lxKbTAHHBkrQpyvR5t+D0wWbJnfM0WVG0fHHl+sYjwR38xsXPD5i2PX3gNRLpbjwx9+TzzxxJZYc8SiWL4M1RoHL/xhw/IGUzfeu3ev9DK0Cdinguur1pNwGqBaaKMev/zVA7Hxhz9TMxoBknhKlN7eepLSNHBzyGjcYKJ2qin0/XCbqrV2WSKbusOFAo8P9zu2VRFMcQHfPGRGyoCDRzz88GNRq1ViYMGC+MS/fVLPtfKIwfj8hedHS4u5UKp2qHPSsCLsC269eFIaalV38b5YDDQxGKTFH4AbAr/2WodQxNQn08xxcR0iSXz76i80aD/MugwEVjJzfDjguOiTnA7fZAMSqcFXzp++nE5JsJsNYEiQRcMMk3dmv0zUDcOScP7iS74R23fviUqpEv963nvjxhu/H2e99R+iF+hZs919w4m0eWHMKoeHE4xp6u52HxDfmRP47BtJibhRVIZu+/69RrpS/FCptsQ/ve1UFUrE7i8CX1abKY6EuyWQAk5r4W3VcBMaJX3LBNwjXpK/MwMMCKCOj87ENddeHeec8xGt5Xv++f26AIMrl8dFF34uGkHPj91W/oPF4T3tX3Mp0WAEkb7BIuSZrL1sEkESWKG4X2zVhmtuYhL1Ltx43UUNC3OWFF6Xy3SWm/nnzYIX7NZ/+kYBK3RalPsVdDoBIiQhkBRMKQ6MMaPA116mJpsLXobFuuTyazSsotZWiw+890xNF/uvBx6J5x1/bAwuxRWgc2grwiGhcsIt4tbyd0j7sLlYmIwaWU+CcWkuLz65aUt897afKl4gC2ABKrVivOONr9B7UkaEostIUh8SF0HIb6VYR8dg2gDWCHCEf8/mlFQpuxwzGouxdeuO+PEdd8Xb336Wepx41ne/933a3OVHLNPmgmJiFXL0mw+LmRgek6q20EpF5VLKqiY6uLmcPF8pExZklqknUJc8vkCHQa4ponDbTVcooKIMhR03V4gI0f4lvyA3iS/LQUvm1OKrOHFtWmTXI3Px2g/UKlYeXGRwWqZdYUavvubmeGLTluiqtMXHPnq2qCL33vvrWHX0cdFdbY3B5QsSvUX3XsGHTWBYOq8R2vDublTvOjVXl5vu0eahnHj79t1xy4afyUVIGbbYGl2dlXjzGS+JWhXFnPbo6EKEOssUulwpyX9Sm4KDOUGTIsfbcgF2OKBIWG9KUcbHZuPn//mLmKtPxRvf8IbUUdgS73//h3SgB48YjAsvPF9Wg5M/OQmpPYMQHr7lC9Ou95X0RJLzh+gAzSdnCCILJKYIBEe12Kg4Yw4b0XbhezdeJoKpBKoS1CdoTwCCo0bTXAx1wV/i31lA1xYdXM3MGZxYtmy5vlRISjrZjsI99NG12Hpc+82b4/E//Endbx8/9/2+gfWIy9etj1effFqsWb0wquXDCuYuS1ZjbGzEgwwFcszohCoaxxUkAp2Ck9nZ2L1nf9x4y13KYXl+yGadHW3x9rNOjo6aOwlJ1Ui3yMmbIqFi9JdkjXItOKdE3GzeTd+XgkP2GZbjw799NO6777/iXz78fgWBSsPrLfHBD3xYF2D54PL40kWfU/6uOYEauGUwiD9YD7+XN1nios/4O8CLbFXd7ul2HPnYeSpJCY7MYtobvvM1Fw7SjeNLpP2oWiKVHHOVMMVGP5gdO6taJhvFz7Ix/GyTHZF4vj4YIXpNxl5VdKjXY9vWrbFz1+7oW9AXq1etSrpLjWhpbYsvfXldnHba6XHM0YNRZZZ6fTZqKKWl5J2FBtJjE4FNSSF4BoIq/h1RL5750NBwXL/+R6L4SNuqWonuTohqr1eQpzE5CZhQLFExjUc+HCy3DMo2rk2kfUVwqhaR90LE2mnR+NhMPPro7+Pee++Oj3z0g3JVuVpWiNb4xMf/LQ4eGpJKzhe/xOY6bWlmESmdA2RRICTucpuyA8wzJp3Lpg1n5JuQQlJLeGtGEVXUIYNgzTMv+tb1lzdELEu3zISvurjJuYubB6VAQITJy2fmXyavZTOc8z/8APnZMwEAfoaH1dDf+Xps3/G0ivDINbAR9vdtMTS0Pzo6++Orl18fz3/+i+LEE46Ovt5296zOzcfY+IjMMM9AoLFr1y49LzeFP4JPJR/EcMS5uH79D2OCNElcq1J0dVbj7He+VpGpaLbPaNfALTE2tRnYlK1Kx3OJz5ZaJ22N2eCS+oX/56FH4v7774+PnPO+JJKW0sAW+m8744Mf+FAcOID240Bc9OULFRhlSyimadYdyaNuyD5IdVJ8kl3dFHOJ0ubx3NxAbrdz4xZRmIztG1coXL/uC43FixanvyBJt37gxOh4MzJD21fIVWpUyj+DKRMMl6JHdc9J3dQpk4YZzjvvhVVpAe45pTPZd6xYuSpBcczEm20qqs3XW+Ky//hW9PUviBe98MQ4es2SmJocVx5M8bqvv1+5ImU81E8zJJjn22rTWgpx2ZU3xvikc2Heo6NWjnf9w2tjYGBAZpDDkE0iroaasTUmXIwXBJjqymQPNGMbu8ViFOKnd98TW7c8Feec+6Go1gw28L4cZv4ft+nBB++PQ+DLldZ42d+dpMNoGo/RN2chs4JHczpJNI1lMBPD7gydL1nOJBHhHNzkOy5HTk1zbb3ww9uvkVk2m97SBsBvEEj4ZYIrC1dZOlesjIQGcdI1PLnOdBMYjjbdImwn9XFVh+iKB/RXw/G0UhlTbnoNKzKmrLtL0ThkbNU4pTdYjFtu/XHs2j0Sa5+1Ip573NpYQuNWgd4cZueYl8ULDg8NC3DRxJOWol6WA3Tpf9wk5TWX7ZDqa41/fMfpsWjhQhcUUrGAzxHe3Eb5sqbPW7DQ2sduxmqJuZiL+hyTtCO2bdsev/zlL2NgoD/OPOuNCTU6zD3m90QFKrXG44/+TjQluNUnPP9FTUvDuucoXRutbj74U6bLQDLMwJKxA/fdUmVTPJMuE01meUPlVmCkAgPf/O1LG8pbi8U09jONziYNSAiQgHFOLLhvKv+7aE7EN5UI0dMKdAjbJUAy74ZhiuGAC/v37dOpOzR0UH5xQB3mjVi5crXnrNcdWec0h8NGGsBz7dixO27b8DPJNKxZtTxecOJzYqCvxwBDoSGUxiqsJT8PEa0sSktcff2tsWv3QQV+/FxXT0e84y2nRnvNIuAq7Kfp1ZmI3tVpojqWplgmYkW6ELEXNDL2xYMP/k9s3fqnePc/vTOetXaNUi+R+Klli9xgwoIGXMxOxaY//EGb29PXJz3NCKNSGVkSMKHnSHL6Sf/ZXRu+eNILQY4idWlYEcB7wkXE/0J0MFkiZSwbbvm6UiE+XKdX7YQ8pDX5M6OC28xXGHpM83VSasAX5bxtfHRUEZ/Gqul0hczhof0H3Cg8NqLvGUBnWNCmF4XwP5vxjGKxcWywI/Ji3P/Ab+O3j2wSMrSgtytOesVLY3DZgNoz84wizNv+ffulicjNvOHmH8VTT/05oOEgwQBI85Y3nxJLlyz07CECFkXiHtki/i+pk7oIJ8EtY3y8Hps3Px2P/O6R2H9gf5xwwrFxyitfkVosnX6x6GDxuKrcH0VHYdTnYvOmTbF3755YuHhxLFm+QmVToNUsKvrMejgbbUaFZ0mII1ZG/WY8GokNSVsMuT8xjBLFhGRhxjO5T4HZxtvWNQjtnfySOJOv1mNijLxyRo6ZL+MmiPGnNANtf1daODHQPkZGhx1AJVOjIQtiNrh8dnD/AZnJp57apMIzs17FhNQsAKcCsC4PC1t6OHGOZvUs+Kl6Me6661fx8OO/14a1lVti1crBOPGvnhOLFvZZh3K+oQPWUirGLbfdG48+9oSCp7KgvEac/a43RXt7RagVNWYLiZiByEhyZtOODE/Erl0H4v4HH4rZRot0GU983nPilJNfHgWaxNNYWuehXjv5SwIhSSfBSKEYMxGHDhyQ9GJvf3+sfdaR0TewUNF+FRVb/qRYxkmLCW6sOYdeGYrIf1PNKpHgVakFUcHTUF/dbgY5qmEvz1P8zg2XNUgjFACk/1PxeCZFnNPTCjLc3m86aW7r5ws8MIl/msqaSe0ziSVP1If/kq+YnY3hkYPR19sb07Nz6rwnt8U/sHnIy7LP9smHU65MAlBRHpI6o8BLlXjs8afip/f+XLVllSaT9tWKFQtjxbLFcdTRR8U9//nreOSRJ6MVamylIhLgmW96paJmbixMkvGJ6RgaHonNm7fGrj3DcWh4REEKdexCzMfb33ZmrF69LOp0GQ4P+1A23JFIRQZlAJ6b2AHVO7olSf/w3+PjozGpQLIeB4eGtLldvX1O3yq1GBkelvqqAynPeRifcPus4omkLMQl0rAMNQiYs4YL0ESwkiFfsgPcJT8rct+PNlzb4Afk75LtF84854kY0l0SI9+nRYhKChRcS5yWL0PpJRf7lRql5qYJlNLA/xJTw81VrarScCrxTwQ/mBjXfdt0ewnCZFoCQjf004YgR1NZ3PRkxAzNw0I89vun4le/+u/Yd2BEFFVAdkjo0xPjMTKG+KYlhSptJXXnVdtr0dnemdyCx8qQP46PjcSRR66Mk0/+exX2uzraBdxk9XLl2ONjuvFoOrqFlJ5mw3/kwNKXFKhCkDop1/Loo4/G4LLl0d3fH30LFqZ2FNLK2ah1eraBGNIKqtyPxObxT6yBOh9Krt1ygQj+ZmYxyw3JTOkmJ91LiBbJLF/d4C8ymsQPE5TwwDnUzqF7ng59WIoezSaoLdZ9EvICZ0opkDm/+NIDB/ZrkdCiYHMo1hdLPoGUyCRmeWhIL5IrPlwFctHRkbGkUwFGPS3qjjr20sayoHwfgdzeffuUttDMzHy7rduejsd//6d47InNWij1KVGlqlkFtbenO444YkUsXbIoBlcsFSxIZqIyWuqwAOxQc7OYn4AJM+IJKwhN5dE6lSKCuiSDT01YtBgotsNDWhcmZvZ0dUWlo0NaGD3M3hOhviwLYL9tK0umoExl2sIzEi9VvEOQ5uY5U3Psqvh+4Fturoh8muEwx829RpubqxvGUQnL3VyEqfGwB7PrXSR2S7xqt3Nu4xhHuoAJI2XTS1XCam8P+nJlRqYt0FVt7zQlJ0JBAptp2g7tKM4x6SVS81MSW8m8Jvtg00fZ5MzG55Dz+2Ojo8pn1ZBcLEZ/f1/87vEn46bv3hlziWRQrZbj7We+KtprzL0jf/cgDMaxuckNpqKB+tzsRlDIjdHMwVZ6ZtubFbA8IZRnlLYI8QkxiJreXBvn8D700EP6zGfhcxcuVlGBdWJNxS3T95qg19vTE6Mjo+4lKhRiYmJMLitHyKwxPz8NAxVyRRInEx6RVNflyu/4/nUNpwKOGo0+ldy1njbSXXyT0dPd08RfiQp141tdUHAJqyDfZoTHCTobAIeI7eS/d3T1aFEz+Sxjq5l54EnWeeaBC88ug0GLLSlwy37fOR/QY00lMZ6J/wZahZlHh+L3m7fE+pt/LLVYNg02w1mvf4Wk7TmhC/oXHF605AoyzCi6j6QAXUGy66H86JSNnRH1SCPXSMtdjnMBvxAIkZC3c8sefewxHeRly5ZJ3ompJBnBM+m8LjEyPitPK+O9jdyl8XUMt8Q9JgQum+2WBP1ijnN2I+xiw/e+oVRI00USrswLQX/hJHqzHWwR4VmTsBQzk9PaaPfJWNBSjD5pJxrEyKeLi44oprvIXcpqpYEYYtgU/gXGR28a4lhOdBObIwSpYXosXz6oRdVph/SOH5diGtrP9veMcMkN1L7lEX/asj2uX79RM4ow3ZAR3vLGk2NBX48YFyBebJQygtRZyHPlQyuhaoECk1FG/IsbpizBtetM3eX9XTFi6IfrrUTuQ4eGYueu7fHnP29XoWLBgoFYtXqNY4pnjKXjM2dnD/O13PSGtZvVM7P2bDzfkzMSXtB5r9mZIlWkdhqdve/ftk7CntZhMlFMudN8XaaDG+HOOn8INwkTNDPll6t1dNi5z1helg57T/ParxuEBQCtgYCnh+toN54rcQ8qH5i8aeW9+Hoic/UJUbeEPdneEdMzs9HR1a3P4/+kFVWvx9Nbt8TY2JCenTRKQUnDaZCCOGSO9gzFlVffHLOzNDF7VuBb33RKLOjvNX010XEzJouLyf8701XQ3RodH9eBoPKFRSBG4FBhKgk42Qz+AE5QC2YtMJuYZ5rQsXwwOdF+ZFwbMw+wYrmbMo3A0lqoDZZDQnqW5i5kIiDfAaae1dolsq3h1VNRSoEUtCDVC26/9evKMuv01CheM43G8GGoXkoqMzo2lpqumU7t+XI2l3BsXaVg06xsSjdCi3wqEzj4IBUfCLCqbleZnHYw4LFtHneDNJE69hoOXGBacuMWLxvU3wkooAsAxZiWhroKDu3fqwX00IqCfBMBjUjlEVIE+NJXrxEWTPN1tb0Sr33138aigX7dnp7eHk+lfuZYmaQU0GzLSOU4aTPPQoofE3SKj7ceh0EgWCMc7NxkvnvPblmamZmpWLFiRezZsycmJ2di9Zq1SQW94pl8Wk8ICGNaK/hboHYcPFo7ucGkThwk1qVKayvPqG7DeTFVdVHSbCYCOG514bZbv96QfN9s6hBXl4s3iN3XeOxE2+BUOWWiAbgqVr8rGqbBajLX/NzhchxMRIECDtg0gCn5Z2biEBTB3ZIgSRUz5A52kQUUEbTE0mUrolRp1wnmsPB/u3Zuj+VLlsgXDQ8dFBmAiJ2WUz1zjheQMxwbjS999dqYmmJzbYZPf9XfSC5hydKlzc3NN8j8K+fkHEKicvGKxdk2diy9S23iaHM92FDPyE1+uqUltm3bpjhg6bIlsmQiRczXo1rriMVLl0isjc/hUnCgodlyqYhNSH/yHgguBOCgo099wh7Uwd6w2ehYyXzTAqpukZQK/egH32wQfCCK7ZGqrmwgFol/wCy7pAdpnYFKBvbVPplmACFVPzk+FiOjQ03mXSOxKTVZKyFgPCxiKSwewD/cXVIlTIq1lezbuX38gU2xd+++6O3tiwWMnSmVY3j4UGzbwqTK0ZRSGVVTdSXxnXNwtnfPHvGtL7rk6hiHAE9Nt1aON77276OnuyO6OruVbuUSYq6aiyguVgcVGNNo2VTAEw5Ppv6Qa2fSAK5LzeiFFo3AUycD0OPmzVLR8XxEZvC1Rzsupr09uvv6rZ8soVDrWWb1VQ4xt5obWyqmeYe0ZqaigQ5Z+Dl5X12e1PmAWebzCxtvv84q01RyZv2DmE9aDjlBubri9gfrL4HKZFmD7m6GPpVidHgoEOFUHqiHddqEjzKDz+aLNou+3r6YmDStU4A/PgNp+QRvZjl4V6sKMToyImxaJjCV3FRAb3MBPleVci2aaJzAj/RsenI6rrrmO7Fv35AWr9LeFm8+46RYONCr4I6xdsq71RJpRgPvw8GSqjryQSnPxP3kMNn1aW5Ym7oSxemer3t4dDjARBrxiSd+L74W74H1wMwuXrJMm00Kg3lljTHzWCDiDYInngn3oui/VtXPo1qQSREOpDz/QD1PHB5RjGDLWOWg8MMN1zcUfU4YhalWs2RBmyoZqndi32dmFDFax8H/vmrVKgU8nE7aQPgcbjc+m6ER/KxUv0utqojwOcNDI3rR7p4+HSL1xSaslAfUYsKISMLRmH5eBI6U6pjpZuOTKA6wocg9cMoB4zMZjxvFIlGd+vo1t8SePQeitchhKGlzV69y9K2UqbNLv0daBJpEn5SxXbMLCfI0GmZuTsEj0SrP5XabOflVnotJ1QSMOYXk5hLpT0+66lVsrWgTOey8oyR4+bxWV+TIubmPE6Muieb8Hzkl5dCoywKIpqZ3flc/l0qcUhdIbZxSI/jB7deqnlsm9ZGMgXtmM5WVxbfAiTk+ueyX/S0zB4hgDx7YZ1M6Pmo6ykzq8puDZmo/ygJpUAPiWZ1dghA56USlvAiHiWcxO8EFB4PklN8mhNbolvFMw8CMlngQAb7FVBM+mxuH/1WHw/xcXPftDfHHP26NEptbK8dpp/x1HHXkGuXHGfAXozM1YTGjQFzkxPTndmINmmPNyQogzjNJLJlVzDC/Q8CIqYdnjGAKPT0QCowh9zsmAI/u7oqWNHiaFhxuGpNVsAZkEE2cnxEFne2yXnxOphflg6XZSiVrhRAfGAwyXaiwccN12lxJ/qlTLaltq1hBEAS1dNbtkZySFNXx5STkTz/9tDZFJbaEpQouSz021n+wbgU0HfplFfEy/Cj142Rcm81Ca1L549ys/HGOkPlsQ42AJSbzyYwnoJxIM6dAdM0bGTKRbf3NG+JhigfFclSq5Xjtq18aRwwuEzKE1jO3hk46VWRa0GlEms+SBTyT2jWS7D23hXnCfC8MSt4d8y6LhRJrqbXZ6QiyhDmVel6K/hcvXtQkm9N6yrvO5hl+KdceOnioqSzn3Ns3u1atyAV4GLS7JKgDtNfod3LQyppyqNRk9pM71jcUrRHJcaWhTKcubhZT8gFq+rKqKTgmL030dwA/WCzGEqY+J1CCk4p5pGSofLlhMRUWmsUktREjY8awX4tm1jsyNDF7UkEb0KF8qDr4qBSNNs2w5XksmUuuqQJ1KnNxczCTkN1UpZqdjTvv+mXc95vfaXOrtVK86XWY5RVC1fge4gFcjiotGlPuIIqCNdEAABbUSURBVM0d/XMqBJgu6qpLHqRM8zQ3QoFouU0XoMlWEYlvWN/BbWMtmUec6+ZYLAAgLgUVslxb5u9HhoYT1OspYNSgcVnkvUpBk04W1tCYdsiicYDYD/oAhCXc/eObGrzU6LCHBhoZsY6gJ1TNyexyQlVISOE4IAaBAD2uPLx+D5nAJH7d2e7wHCK1JmOmP5xSBQsT0wqGqM7wObkowWcoqFFXG3kzAV4aClzA7E/osPC9RoscjMkfJq0qvlcaWbiHej3u/tmv475f/4/MIHpQZ7zmFfGcY9Y2p2qZAGhMnRui9IIuhMQ8aZK/a4yaNWsCF6PJhPjl1E1KCsaaZXUAigbktlwOglssEfEKzwqYQa8xmzwxnuhJUqdpUf3Wz+/OyvaOmkCLiXFST6dDKpF2dSZKUx7HagAqm+zCxtuubUA4U7de6tHh4ZnHQ95FyS+T0XUTE+Md08HJJj3JPCDBkcm0gH+yaQQVbCY1W8kalK05wbRN/DZtKJhgsFaERa2A5pOMP5X+MSa6ah8q1Ep9QiZx87N8ftauIhd3Yds5M+yEBx56PH76018gO9Pc3GOOWp1Y/Zbpl3/WVBWoqhDc2bSGvleWgRw+NaILMxet1oeLw8cV5pYqF9btL8a+fXuULWAJMJOlkgMp+fO2imgxzG7AikkFr4T2FNWgGUOzsxYUHVi4wC0kRRrCRoReYeGUz0qm2IcOK5lr7QKSNt56tW6uiGxSUTMfGefND2RtX+G/XV3yHxq/MkfbBovvcZ/UGNlMugX5ff5uYGCBAAX+XYhUyco05JWYOvxk9re8LFSUFYMrtIh5Srb8fr0uU8vva4FTAJb6SIzyKOK0xZEphTzfUlCUvWnztth4x8+lD9VeadNQ5qOPWq2CvFV5qFsTmDlfHJ+wcCdrIhQOfa4K5UKvj2IF/pnYG1kpVlyq5hQ113Kh3sICEZUmjRbg+VkD3p1Dif6Vs4SK1g31G/5J9N2/oF/rKsL93IwqZgBIqhCJmOjxsLlIo9IfI+5gtdx+01UNHlTkciY9T0/pJbDbqtWmEWpgppg9FlSsANUqh5tsR5JmTAk1RuWAMDiqvqXudXXfqfKzlpYYn+JWm31AwJXNK88gwRJySD2HUSFH0yjR1eSP8tjyzH1y7Rn9qnKMUWZUW6VZmVu27IzbN94T86inVtri9a89OZ619ggtlH/f00AUcbZZsIzZgZDb+cNz4wYyW5H3E9I2Q/VrXhi8GSl2I+aKjem9+MyhgwfVuEYBQuVVMGg40ryLND1oban4QAtGNCsTd8MB4zPU1oK+c4Ztk1gJzwKnnN/jebAMGV0rrL/2yw0+iEWkIA2tkxPVWkpkscRJxs6rFRNtjNmZGD401AzXVbgumB5jnUTnhKQZqN8o0k0142oHSqdm9GFynQeXxUUmGdcMPoh5pFJQTsbHUzqUhFY4IMlcsoh8hgQ+U18u/TR077tWjFzgXBw4OBzXfnuDikgd7eU447ST49nPXit/B0GPeoNIgYnwRz6NOTZfuNGk4rKAgBM8n/JgSGozM7Fk8RIDPLPwoNu0KQaAxnQBvPmHg1MVMcDVISdAjk8HyikodCbq5+afsZZYpOXLlse+/XtS/m+oFcwf64T1JLjt6DRu76rcPI1g/0Hhvgkb4gsFBMhdGfznl0FLqEcafpyWWVY+q2L+XFTKsAQndBswE1gC2i37ehfIR+D7+G+M9cb/8gCcXDZH5lyi2I6cMW/4YPwr/zt3OWS+s9CX3EY56yhcwpzcQPlwgIVRFdXZiLHxqbj8qvUq2NMr9PrXvDKOPmpVdPd06X2klI7iqTBZuycOCH6QzccE8uw69OrxBX3iUIIBgCpVNC0UdQJVo5JkPf2+BKLqK0r4vNM8V+DUFZCmfmEZ8b1sFg1imbGCe+Fmbt22NU488a8UtFIlE3Eu1ZG5CHwPe+ZuzSn3Kt1zx/oG+DHSckqAK20xMjwi+NHS7y7z8YCSYAfoSMEKD5CpHtBy2KQsX8CB4cTNAFQgTZAFzMpuFcUnyMwrN0Zr0gVvzNMzhUSVYoB1p3GmPKPUbkQgBwefE5abu+V4lwxDZiYH7aSXXvnNmJ6bjc5ae5xx+knxvOOPU8O4ABONN6cwgFAZ07B9gNlYECV+4CAdAxqPaiDH0bnLk6RR5MaZP01hgQNDmZPn5fMsvOYblf0jvw+9lwMBA0VdA+pbsViYg0RPK+OS8d2rV69OAZjnPYkRmuYT8jOskyJ+JBju/P51DW5I9n9snnxtmHknjk4i95ASiNVHYFOva9P27mNqdD21QtjJW2mchUAjAxHrsqBDLEAWDRPLYJxJHER+0y5u1+uxeMlid8qT+6b5s7ycYUVShDEjQbWanoU80XRc01lIP+Qni8Wm3j/v9rWrb47JqWnpVrC5xx93bKDtyCIqqHNLnosPIEoj8KvT32emBV38siZT2mBMtEw5Mx4w11Kha6gSZilDSxCRcbiH2CCDLo2kkWgrdeVJNeS5ui6XJSwazfIl78UBIPImQqbFhmc21behAoy6FFtahD+INz03G4Uffm+dfC46URrP1ki+B+SjvV2LTGChoKK/P9UnZ2JkaCh1B3DLKwyttp2XfD6pTJKfr1QVGWaVG5iMripZ2oAHwrSxsZlhn6G3zM/NVBteIOeY7p4vKlDh0FjiwBpWmGS3WlhGmFru+ps3xghuo1qNN5zxyjju2GN0sKwtlaT1lZPjsxz0cIk46Ji9PAk0u6E8UlWBI4AEc4HSbSaqJd7QCDlx0uichPNl2hAN7XljMiHfgaoRNeW+E+M68ELZ4I436jE2OiGXNrh8UGvIcxM8Ug/gsKnNBzHwVPcu3HLDZWonQfZGYAIYbSKa5xPKqZHmRAsC2hNaSGij/L3lFoxsGQCZkpnCd7Povf2kQ7Ni+OE/ANaJeuH+Sje4jlYzaqvm3nJjMCksZmZdugJigS9utZuezMbnc/B5SpWkB+W0hufIbMThkdH43oa7Yv/BYZnlU1/1sjjxhOONmlVraeiFJQFznu0AyFG7UsM0KMIYsNs+RGhAOYD1aLOJZvNMKSrHnr27UzCYx7p6jSgQqBU0FUw0H1gTOU1Sz9RWK+HaYnGTWFOlZ4k/LnKEqnh+dtZB+5GKL4XvfutSlfx6uo34QJPhxGjiJGYoKZtjfkTZbHNHGUOK+KNgi2qRBld4Fp279ayhAcWUm2tmR0OCIiwCP8dpzhsDZJk/S+aHCJqaJuYt63AQjKQWFx84sz8w5Rw6PTe3BTgvCW3y8nv27Iuf3P3z2Pyn7dHZUY03v+E1seqI5amTD0Idcw7Ugq7/lqsx1qZyWsc7a7BxCub4b1g2UYjwwzRsl+wneU8NPw5G0+2N/t4el/hS7xWtNkazKNehAH9Yqt/iMEkLDJl8kdBbXK2qeo4SB1mjC2ZmdZMXLRxQCpvLsuIyo43xg+9+vQGg0NOdwPZZ837yxAwiXYMNANit3HkHN5H4wm0VN1fPz6ZNc88RD8Qpw+fiF7mNKjSXHXFyWDT3jnHj1HyroDcAItZZ3rVjh0VIkuRu3mTGsuB3iU5lIUqtSnl88tv0ghxCPpfDIS3L+fnYtu1p8ZgXL1oofefc/JYBBU0laQDeVNxUJZSL6k89Ors6zawMSzaIvEBUm/5bE1qdI0+uqILDc7MBkA0g1hnSteAm5D5pVs8mi0BTeHd3KuclPWWBIfQbt6lLEUvAuglyhaCYNKtEL4Luy7MDgkyaxcEeFb7/3asaon5UqjE/NxUVwPxyOfbuO6QPypxad5Mb8VEHndKO2ea0TPpbRCgTKX1GmC43KwuFEpxoUYqMPnPNkwdEUR1zKr4Vc4d0q6Fvply3XI6hYSZvesw69FodPjjEcLGUKszJ9zoNAwI06x9zevAAAUZLTI5NxM6dO6X1dOxfPNdiJ4q288icLG1rPUtKb6brWthbqujphvFeWAm7AmtTShoiTc4k0maRuU1KoQpFkxHqNLzVmmAJUGxmjuaCgipqUiJ07EIAxedzwZQDZ8pwCYnAMSNaaSpLHqhBYCcU75Zv2+eS4bfXLJgxJFJXIqmJWF0Q/0hOPA1B5AZqISUmYmFP/i4XINh8zFiudsAOkLYVJK+k72RTDCV2SkEQn0caBltBvUqMFoeNkIY8kI4YurTgtiNt6zYtXrxYFoPF5r/pnRqFGB4ZijHoP2ma9MT0dAwsXCQZImBLNhHTyB8fNkfuagNNcKclAX0480Jy0zgYmr1XYrxOh96BzVLcAGk8FVKgDfP7bK6bzlHRo5zoxm/HG20284yAt+6g05rpKanQcalECKCtVKPRoSGNmZHK/GKUBZLwJ9i0yrN3brimMa9RMo5iJ6cJu8ll7azpz2ER1bmuxBnkaqYJcuexLWMjI0ru4VHl0S1EfYw9E7pFGkRFgw7C5Bf5XMavHjx00KnNMOYdApmjz9z1l2UQ+H4WgBsIMsTPCQgoGKXJz5kpOyr7UcCQSAo6kvUolisxOLjCOtFJ/d2AhNs58iHFxzZH0rQU3cVPDt7uMiDP6/TH7smYMwMT6XsyqyXTktRDRGNb0p7KBwXGh7Fot14KXZqjsdwHmtZNU409CQaky9zlqqwZeySCfxqKicVwwAeXqxCFO25b16BLDJCbkzIpkjhTpkxh1SiXlLIIwEg6g6UKi0pjkiFAZHXwnUBnfKH6SVMEmIvoMtuopSWZPQ6Dos5UhKeFgiNJ4AC0xkLysnTOESRJKzHL86DRmCJsPgPzxz+59SJwM90D38lgyL27VROFHssc344OqkgGMHI5jigZ02cEyVIPCnpEyE8Dq8TOcETMd+WhURnUIH3Jne98BrFBDvTkPykgaJiFh1th3eSqhCdYicYWxN0eo2OkmW2aPsIBt+BbMbq6O2Xt4K+5R9cDvjj0lntwHl244/Z16hVCdAlucmb3WafRRWvMDLVD54zWF8wFAV4GIhrmkmBkZNgMSJfeppu4qkB3JIY6McNWUc8+UwyNEYP0+CeCq/zv/u4uRYbcSMF/mC9Mb5rbx4HA/+n2JhNJ7kxn4PDQUOzatSO6Ozv0e/CW+gcWGu9OnRGK8DVvwYx9ntOS9qb5AkMS2WJxGP+eSQDZTCu9STPtM5KWJZ24YULoMPVJYDyPhqFUJxeSmsZUoUqBFs9n9UM2q9B8P9aWvcB8c+j1LETXgpDdiUk+zX8r3LXxOnUcAD8SfeamKkwri2EqhyeRYMZ4Qb5AdNVUuG/qMqmDwDVFtXaWXd5zv4uDELVTarYdBG6CAksBI1oiykuCOMXWmPP0Tke81q/ys1js2lHhdPI7DvA0L1Cy/M75YPtPjNGKgV8rxcCiJdHd25fGh5uaYjw24dg0UqcAL7NDOPtiZUitzQ1kigcm7dsx62w6SjtKU6q12LV7t/NsjYvjorRoNCy/i5Xke8GS5VqymoEOHBG7LR/mV5vFDIZED86bbvlhsy05ZMIESgzlcoApHZONt35DHCqxIzBtdWCxolCObKJkpkS9sciYyGeahuk5PMKfk1wdneT2Xz753Ip8M0lZMHM8uEd7GxtmA+jqM2mbQcUz2rgsLsrpxiRBdQHpUvlRwzNGtTj8nbrTCwUR0WBG0p/Li06Mj8WhoUNacFRaeQaKF5L3SXxk470ukuQcHJNOJI7LOFxzdu9wVkf34EZbMQ4l5lmWrdASO3ftal4GlTWZ51f1QCzgRQETDbdioqpn1XnHDiBYxu9dm6aq4UNIL/N4dLTXRHQwv6oUa1avUVO41NOTGn29MePNlTmE01tpi0MHhy2igYNPPoAH5uEpJpgh6ZIYZpLNEPUFdGl4RGUn56QGyHHyHBznaEzT3qfbTKSMj+OU6vDMuWtcdNqKzXKT6ZEEScxlcnpln2agXBpUiZBNtC5+Un1em4pwda4mgQANDCwKRsRiBbKgadMMY6068O+Q8s0CzRYqayCb0+TAB542lo3bSfmRxVfBZHLK6VuS/ssDpsrFkpC3fAFoDQWpysBOzoPhWlGoBxThgkh/szktzP27fKYCyFTrzmgeMYFr3fNR+OY3vtCgDYKolgdn95XfdnQ2WwxZyBnEP5SSWEzSnF4n3AQO8H4oKM/XvQGc8BxI6XRmFXFLs4iZYdNpk2UFUg+cYvNFwk5oDw9LZKiBFlm1NHG9+B0FYmoGo4vfpHIRBqbcp7Rz924dLDoF1anfXhNoIHM2N6+N4Rk7EzmdjVUaRzXo4CH5W8kEthJo2mpJTiiRElTbncPiOLfGenCYPSDa0CHrQYEAK0bUrJJnB5TVUYEkOd3LLJNML2Z9BHwkcXK+k0BUUDGYBDLEDOVKBRBLSxgdLGy4+WsNMec0fwdFVeeXLZiG1FKhwGfCqBBjx9lcggwWxCquaC5ZvrelleZjK3xnOogWYQLNSPsu/vDinLyJcZt7KJsEb4YaaRAz1QCTRhGfQY8EbmhLqqyXGr/4PE454AkFDtRyNAMQHHxsLDrp6B8dFXHb/F7Pn+WQLBoY0K1mQ1gkNj1rPdpfqpimm2PL4IXjv3taiEuiedo068ZaQB7UjSvZWqkIgPYkHY6ow6kC1lAJMqvycRg4lCrCFFv1rlhTrCaWyMwON4nzjBqCOQWfzFL4agTAwgrUqMbBgweicPePbmhgVpjVqmoI0kFJXIwFwAdgkgmm3AnuF84Do/wAU2kaJ7TLaZPKmJCZ5guRoI+NDqssiLimyndpOAPxqPpl1Id7QOaSPHRYNWZHilIjTdLEmDJTbxzwcbuBFyGBa3R6S4u67+jrwb3gv4kRPNXE42UkCNKaBjbR2Y60ktI2k7o5hXyulGmSzgS8Zg4pG2BV9JaAg0wzmJqnobKOuK+KYrveKSmYYwXgUmXdK9bBJUwiXEJi0rRMj/EUFck/iRljsRlubhYQB3dXNiNgadqST2hRSfGH7sY0nu+ujd9q8ItZgr1WgaNUUBWHm8uDiTucVOMI43MuxemUlpIK3WmI47zTFZlthVvAjCTX7taHa6XitArkMyKpQ/NEPk+mCnAcjFhyhPivGUn50R/rG02JkGDCB0/MC/F+DRtSz4Xch0kmAlapDYgQacCOTp14IE82OLNJNCkk5Z/qOpDuogNCddTjqnAtSUmARjUzMyk1eo127NgerB23lGY1PRtq6m2VWLCgPzb/cbNlkWh2SywSUhbnu1YI4v8jaOQ9lZ5ChxVo4oBPaBaVokSSZzyPhdFyPp6HOnrIRuGeH92gwgEFYTdrWaJgaoq5NvCmKgq5McFWaHVFBxO7bx8N1q5q0N7R3U3x2qWwnOBv37lbYHtfT5cgNLhD6iJAnHtyIsZI/KMQHTUDFckli5bD7cC3YN5dv2yRSKc62ATbeYgG1oQ2lozw8PL4MlReVZ5MPKtc1Oef8Ke5TZx0eoRwK7kBDTegHJcJpJWKGSipiK9iSB79ngVLILSrIR1kqaFigdpUwu0veo8US2Ca0eRyyykxB7RWi5Ga392QTyUv5tmZOk7vkGYORZaFSi03PJ82mBiDuMXFmQyKKFpW8JPSm1yaYnMV0GhwYVUQoZulLf6ZKaT4NiJg2JBEd/wT3yzuVa0qnrLIckWzENRjQ4UEuSIA+rlZLcDUuBEmtWOSLqWmM35HeCr4aVeXhDU1NFFj3TxnlvRq755dnk1QqcShgwdlbVQZQd62Qk5MxwAqNHy+5/JZbaemETfc6FwnFXcqcZ4wwbikLGBqQoMPO89gfShbIUiC/EG4VNapUDThoVySqt2ixYvdqK54hsoTjXVzUg0Q3AiWLeTLBIcs3j3RBGhMoNNUtukpN6ylgIv9A2Qy6maK7v8BHX1Jnb0Jj5QAAAAASUVORK5CYII="/>
+        <xdr:cNvPr id="1037" name="AutoShape 13" descr="data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAHcAAACfCAYAAADDLkZlAAAgAElEQVR4XnS9B5RkV3U1vF/l2DnMdE/OmpFGWUIogBDJYGywDRjbBAPms0wyIAMGRBLJBNtgMNiYbBwxwQQBEhJgkFAcxck5dw7VlevV+9fe596qHsHfS1o901P9wj33pH32OTfYt293BAAR4mhHbaCtv+orDENEUWh/Cdr6FrUDRFGEdhsIAvuz/gfQaLfw8je+G9VKHWHYQKtWQ9Cu4kuf/Qfkc3m0Wi3s3/c4RvszyKSTSKdTSGUyyGazSCRS+nsQj+u6/v8oClApVxCGEZYqNSxVa7jxHR9DaW4aV150Ht77rr9CrO0+H+N78CuGCAHufXgPPv/f39ezx2J8vwixIEAsHkcsiBC1Q4SNGqJWC41aDa12C4kA2D7YxDOv2o7hgQFUwzg+/fNpRLGEXdetViwKEQ+0cAhi/AO0VlG7jQghauUqmrUKKuUy6uUS5s8cR1gv4+tf+SzGR4e0tvEE15C/F2ltYkEMcH9vNJq6F38eRnZ9v95xBEilUmiFdYStGk6dOIZ22EZfXx+y2TxyhaJ+L/iTP3t1tGp8Fdat34jztmzEcG+fe9DICTfSRf2yRVFbD2MvSiGb0MN2GyHaeM3bPohqpYGw1UCzVkU7rOKm1/05kskEfnzbj3H/PXfhkx+/Bel4DNlsBulsVg+aTKb1PZFKIhaL6X9bsACNegOVag1txFAL23j9u/8ec1NTGMzF8c+f/hjisM+22m3sOXAYv3rgITxy4DiWGm3EErZZYjG3KcMQiUQCsXiAKGyhReHW62g0GhJ+PIiwsaeKp16yHmtXrUIUj+HTP1tAvc01iLvnanPnUx3cM9rCt6MQ7Tb/b6FRqaFaXkS9Vkd5YQZLU2cQa9fxP//5ZRQySSSTSQQx/r4pB4VNycZjMYTtEM1GU3rWarYQUuJPEC5/P2w30GpWMXHmlIRZLBSRTmeRSKXRCkME2699ZsQLh/acGBnoxbaN63DB1i3Yvn0rhnp7kIgntDslTO7OiAKPd7WWwg4iNJttvPYjX0C11nBaUUVt/izQrKBeKesRE7E2Pvbev0IqFUc+n9NLZjIZZDJZ/TmeTNriS1NsVzebLcwvLCKIc1HSeO37/wGz0zMoz03gn/7+Yzh4cD/uf+AhPPzYPpTqTUSxJBLcwcVeJBO8Dp8XWnh+j8fj7tptRE1amCparTq4n2JRgEKsiudeOoKN69cinkjgS/eUMFcLEMQS9u5oI2hH2hzOrLnvttnDVhWNWh1LiwuyDJXSHMqTZxEEDXz7v76GYi6NZrOJdDouTe0oSNg27eQ12m2025GES7tIzTQl40ayTdYO6wiCCPOzcyiVSigW80gmU6DW9/b2Itj53D+MKGU0m9o9qUQc1VoZ7WaIdquBTWtW4O1veAOG+ntsQZx59prrzbJ2bBjgLz/5H1iqVE3wzRqWZs6guTSNKGpptyfQxi1vex0K+RRyuQwSiSQKhYJ2XIpam0ho8fkC0gaauSjC7NwCmmEbC+UmPvn17+H0qbNYmp1ALKwjigUI4hkJIqD55e8mksgWiojT1MlYd/+nWU7E3eZsNBDWq2i367pXEAGZoI5nbC/i/G2bkc7E8e8P1XFmiRoWM0HQVYVm1gNtHLtWRwtbVdQqVVQrZYT1GhbnJtGYm0EAau7XMNhrLioM60gkE7omhcX3pWDCsOVMcKDPaS25meT+6FpskzXqZSSTcb3j3NycBM0NUSwWkUqlEVz6e38W0QwEYQvtdgNR2EbMmYlGs4l6rYqoUUVfIYPxkRGsXTOOLZs2YevWTRgeGtSLBrp5As0oxE1//28oV2niqBV1NGtllGYnpL3xRBJB2MTNf/FH6OnNIZ9LI5nKIJfLIZWi9mYQT1Jr+aJudzrhLswv4hOf+xoOzpTRbNHHxlBZXABaVZNbLI6I/wNoxxJIpDJIZ9LysVQPbZJ2yKBBmyAe8363hWa1bO8fciHbSCDEUzclcNEF21DMZfH9x+vYP91AW5stpP3vWC2vTTTpuj4iNBs11ColhJUKanQpcxNoLM0jiTr+49+/KkWRnw0bLraA3IZcSytEeWkJcedOpFDgs7epGwi4nSIgajVRb9a0VqlEsmON+DzJeByVSgXBRb/3/yI+cIz/B3w52gnuDwYHNIkN+TxqMejk0ZIwW2EL/X09WLdqDOvWjuP8bduxZcMm/PVn/xPVahMhzXezLttPvxa0GmaywgZedP2F2Ll1NYp5+lyakiRy2TwyWQrXHpTC9WaZL1ZaKuND//gV7D05h3gyi3gQoFmpIKxXJNAwCJBIZxBLUoNTABeLG4za6GIGmjagLVMtn06BhA20G3W0m9RcEy7DsStW1HDVZReit7eIu48s4p6DbYQxoCk/3ZSZpIAoFC/gMGzqHZu1GtqNCsLSNMIggfL8FFrVElLxCF//6hcx2F/U74Rtu04Qi/TOFFrYaklb+T9NNs1yk5tA+5ebMsbXAtotlJfKilMk0KS5MRNuAtVqFcFVf/rWqM2oOGwibHFnh7ogfzZUSKAVRphbWEIMfBgGC3X5i3bLBBw5oQWxJPqGVyKWKQIBTU2of6MlCJs1mRqa/aAd4tLNw3judRehJ59D9hy/m0E6nZFWxuMWJCEyX1+t1/GrBx/C3GIVSQqPzxO2pBmtKI5DJ6ew5+RZNNsxtLXTTbguvAWtc9QKFXrRp9vGaaNN4dariLVbCClkrVyIC4ebuPqSbbJOB2db+OZ9s+6eFD60PmHQVhBGVxBvR2hQ8M06wLVsVIGFMxgYGkEhE0c+m5FretMbX4u+Yt75aNt49UbNhNOJvGMmiyBCo1FFvVxVrMAvKgJjEH7VqzW9H3/Gzeq/h+0WSqVFBFe/5t2R7VZudpfatNtotdroycRkYqZn5y14UNzUtB0StdFs2SZoNhr0BMgU+xBP5QAGHtQYviSjvVZNG0I7vd1CXy7CjS+8AT35LAo9PUin00qHaJbDVhu1Os15HaWlEqrVinZhs15DIhWXX47HEwhDBhy2Efn5fLYHmYEVuP3e/fjFYwcVkJj9Mn+mNIUuh+/p/JvFCQ20aJZb1A5ekzlehHXFOp5+6QaMj41hqQH800/PoN1O6H0DcHEjDBT5zGkM9OXRn81ioL8X2UwKfX1FuZreXApBImUbu9XCvr17cMVlF+q9eR/6S361I258CtoFe863U5logKgQ9XpN/tSsX0uxSiyyYIxKlkwk5b/lixt1VBjAXvPn71PmRp/DXNDns62mRcV8UWpcm1Elg48mc6u6KYW0toEg5MZoY/P69ThvywaM9OSQZg4Xi4EKKC10L0gzz5cZ6c9LSDSv9A8MJChERs0UYDqTRCqZQiqZQCadRiadkMZxd8oOd/JBPkOEWrWGU2dOIwwTOF1L46u3/hIhcwkujswvN2cks9YJ1Ghdwgbq1TLSQYR0PI6lcglMYEdSZTzzknVYt36N7neqvRrJVAqDfT1yHxluRgZwZgsxPTWFeDzA1NQkkqkc5ubnUFqqKLg5dvwIVo2txHe/+x18/CMfQCwWaUPTlwbEDWgBWg3EYknlurQdDCDve+BBPOOGpyIZowyaWn+mbMsjfioNQQfLMOKSVbNVR50Yw7U3vj+iEGmoFIbL13IHu8Scf1cKxNzOojUKmoJlJBhr1fGC6y/Fjs3jSMRjWCrNI5vKKSBoNBtgwp1IxBQoJXlzhAoapFRRhBzz3GRS0Z38V8yAhg440qZ1sGCIGmf5oCklNw19FXNCS8+AmdlZHDx8EpX0CL56610IlbrQUjYUCctnKT9nAETLUpNwEwyklHY1kIi3MZZt4Krzx7Fh41pF1unRnTh2ekKWJGwyep/Te4yNjeHI4SNYtWqVfpcpyOTsPC7cuRMnTp/C7MwsxsZWYbC/D3v2PornPvsGpBMGWtRbwLe/c6vee+f527FqfBR9vX3S4jt/+nOsHBvFdkbsCcrPfD0/y/twLbjGfHe5TFqUgNF1Uy5oqVRCcN1r3x9RmPyAsxE+PkMmkcJAIcCp6aqZOQrWmQbu+EzQwptefD2KmUBmiClNPkshxWUuFFy4FMv2o4v95OsYtS7LlZ2W0XTSzCYV73Tvx5fyaZG/jpQGMSSS3LGM9tuEAVCuVLBnz0GcaRXxPz9/GO1WXUFiPp3AxWsLuHvfFFq8X9RGWGMwVZOQGaRwYccKIeJRHRdvWoEd521CKpXARK2AX9zzMDZs2IRypYapqWkMjQxh5cqV+N73vod8Po8XvejFiMWZf4aYnp7F7PyC3n9paUnPd/HFF2NoaAgjQ3149NHH8OPb70StxvyaoE2g7OGvb3ojfnDrj3DrD36AN7/5DWg1qrjskgvRDGtSFH7W0qhQG1v5rgIwBq4WffNeCqiu+4v3SXO5q2WGJUR6nwjxCNi+YRiPHpqyFMB9cXeg3cSLr92BJ21fhd7+fqFN0ipCegw23P9mAkNpDvNLRqsy8+22QWj02w7l4uWZs8lvVCtaKJpEbiy9xLJn8IiZ7C5/L+61OpDmz5dKOHLkNH7w6AT2HT2rGCGfjuPJ6zP46d551AnPcbu2moJJm82qnp1W6bzxAuqVJWwcLeLSi3cgnUphutmLA0dPYmRkFPsOHMLiYglHjh7H+Pi4rMVA/wDWrF2D06fPYHLyDEqlJSSSGQwPj0i7FxbmsXJspeKKI4cPWcCjdzIlkEWJAedv2SxwYv/+/Xj/+27GY4/swgXnb0M+n0HCWR2uR6vZlHAFyLTb2iQMGJVtR6EsTHDtje/tCNduRPPGZMAS53iSUbJFnxI+N0KrjVy8gXe+7OnozWXR21dU5CksmiAkI2QXbBHRUpgf2gPRZPA+9BGd3+lsLotg+W/8DP2LUG+lCUw9OvvLmWb/g2464v0p3+HUyZM4PVPHF398P2qNFnozCewYaiHMjeCBvSeRSiRQqzFYo6ltCi5F2EBfNoFsooXrrrkWv/38FyKdzcnvl0oVHDl8FJ//wheQzeVRq9eEDDFF4aoWewrYt28fRlesQF/fAFrtQJo9NTGNUmlOqQ99Kn2th1cN+LD3ovYODw/jJS/+fRw7vB9XPekyVBcXUOwl9p7QBuXv0Rr4oNC7L64989s609Z2iEqFqdBrbhYszcUXRBcx4GAyYJrMpNl7346za4a4evtKPPey9RgdHQEzC2+uqZkyG8zThKhYPpgIYiAowsBAvjaXQ71uqJBezN3PkB4GaIax0td4M++B8+Ui9p+XgQ4sWJJG0DoA2P3obpyuxvE/d+5CMQlsGWhhup7Byfk66Coo3EajgkalgkioXF3mmwWJVStXM+LQZqfLyWbyyGZzaEcBFhYW8Mhjj+Kee+/Ffffej6npaaxZvQqzs7PI5HMGwsSJmScRRDEUi1kcPXZYKQ7jCgZUyo8ZB8g9WRRfKORxy/tuxt7HH8H6deOIR21ksvbvwhrcl98cCqhkuUyDaZ4ZoApyvfLPbpbmCvtwbre7+/kz8580WVo4BqBhiJc+/XxsHMpg3brVDv81oSGyxFwIlSss0AIEMA2uVqoK2ROxeBdacwL1u9C/gMFyVhmx53MPeK4Cd/7mn1vBRtzSAqYQu3Y9hj0zbezeuw8rM3UcKqVUZFAkHTZRLy/JHDNto4+77uqr8JIXvlCRev9Av3JtVq3o3xn4qdDhChzcoI88+ig+8IEPoKenR8I8cOigpSxRHP39/fLH5fKSoljFIA1asACJJLOCTEeLqQCxRIRnPe2puOKKi5BPW3GBPp9f7ZaBJAbyWAzCdJRuyG98Po9wCKbJT3rNuyMFIsJgfQnKBT7SKvMLNCZ2B/PFr372BVjVn8a6tasdKN+WJkZt213LzYV7Mn3z1Q+lJ4pwl0XGy+xuR4MdLGc71LTo/++LppsSUwZHpIYmJQDOnp3A8bOzuGvXbqC2iAMLcTzj6kvxiwcfRbVSQRIRyvPzCkQG+npU7bni0svwohf+AQrFgl0viqucxjhAoEqlqjyVQuYasWrF7KC0uIiTZ07j5IkTuH/Xwzhx4gRKi0t65HqjbIoSWnoZSyakwcoSGApKkVt48R+8AFu3rkeB2i3hJs0tOQWjVVKWQL9L96bc1/ytMAfluk1q7nusQhlZqtFJE1xqQbBcfqFTAVHqiz9/5vlY0ZvAxg3rOr/HB6gsLcpfdyoYDvAW1OZqxXyhSsleuFsL9dG0ic4n6su1WYFZu6Wgi1GxnpsP4x3HssBQgEk85oI44NHH96IVJXHw0FGcWmhg/fgI+gZHMDQ4hIH+fpXLUpk08tks0gmLXlVFisWQSWclWOEibZrUDGr1iqwCNTURTyKXz+udF+YXUK5WJMR0NoOJyUn873e+I/NdLptw6Q6IMjVbTQcEGRAR1htIpYEPffC96C3mkWIVLM0ghcBJgHjCNLQhDbac3UqEbTSoWHrnuFxGjMWTy155c8RI08phVrf15tTySvu7yt9Uf1NqPP+SNbhgXS82bVzfCYDMfDexVF4y/8cd2Y5cGhVqp+VUtG9q9zIg6ZrabrTk/TB3p2BM909W2LY8OU7smT+QSfJglAV83nLI7MaYPsSFjz/62D5c94znqd4ZEg2KMfFPyYQrkg8MpeO2YcZP4bXCpswysW8GUbQcNM+EEmdmZ4QMWZWJ3+nr27ywW+iYolhu1Pn5eUzPzGjh77n7F/jFL36JycmJjmIoR63V8PZ33ITVq1ciGQ+QTlC4cYQNCp0YssmCMCdjGhYMVCgJQ6WPFDTXjvdIJTMILn/VO2UBKWlfrPaLaz7UKjD0oTIeQRvxNnDh2j485+JxrN+wVqaFX1aesjSnWlmyPMwFVDQbFApTASbhUjiaKifg5f7U53DeNC9PlQii8Y2a9aYWk7iuF6bcyxMjam3IQM8yNTWFxVoMVzz5Wkrd6sdErOLJTqFCG9j5dpo7skAE4MQCZJIZ+U+CNY1GTSaQrsj7QAYIlncbmtZq8/3qyhL43pVySegU14km/P777sMdd9yJo0eP4PTp03jubz8bV11xuYIvXpPlVxUGtKGbiDm4kuuYEIBR12b05plC5v2WymWkkmlq7jucWXZUFfkt+5LGsgjggiPT3DZiITDe08YfXb8DG9evljZ64aoyws+HLbEQkuStOF/LQrIvIFh0zntSQyzlEfzpvmgWCSj45+hExYH9XiyKqeIko+wDCqVs50o3csKVBiPA43v2YeuFT8ba9RtMKMq8VXMxN9EJ2ugDabnsPSw6tY1ubJhIQvYgDYVJK2csD4MBCZTwegycmNYlYsDi4pz8Kl0YNwo/t7hQlmbPL8ygulRCb69Vyrxwk9xMzZoqUnxhwqD8A7GD5QEVn4XgRa1Gd5FCcMnL3hYpqPFpRGdtXKmMILaAZGfi3L8n20287UWXYXSoz6r+QkYM1xQUFllKxPCdL0wfQw3nDhRI7gIqL0wrl9nFfZ77xOi5m/bYxqM7MSjTIEtVaFx6YWmYIisnNKYacS3yY3uO4dnPeyFSGSuX8YtuhNiuT/wkaKFBDOQMaWO9VwGhSn3UqrRlCIClHwF/HpMV5LuSXCAWi6vNJhiJAsqN+T/fmbynZCJtkC9YVWrizKkTqGszBDLHRNJIVyLUmMkVkMpkUa8sdqyHXy8KmrVgYupBkEJw6cvfbneUD7NgyV7YUhmmQh631ILK5wDxVh1v/8PLMNBTEKTmgzHuMOZy7dAS9kadrAwjqFFTqAlaECfIrsDMXEkrl2HIv6a5bjf4KNsjVRTycs3z5tlxy0yAcZW6cfrMLNqJIp507XWqk/BaRr2xfNJvKmqpca9oFrnwRLIsN7d0LiMNYQ5MbVlYmNOGYGVLLikRV+GABDdbO7uO+E/U2MV5LJZKKOSLqor5KhEtAzdhfalqOTsiLMxNoljslRKSSDg1cQqlhUkpAk0x34HPQDM+PTuHRJxMjJe+lQVJRIqUCf/ZTiZ4YDbRgAEJgQGHUg0D3d/54iehmAywes24gwctJDcQw1KiIDKckw9v8KQn2PlF9KaXv2vWwtNMfBTstds2giX+ntPl0ymad0uXvHtxj99JjR1MSbZGFOHx3fux8/JrMLZ6nYu2TevFjqTv5KK6gknUpOY00WjVRD/i82kzxGLo7x9COpVFs9XA3Ny0e1RqcFIuIpW1PJbFBwneFT6MhWk0GmLPjHazOUPCvKlRgMRiRqOlfJi5uWHLdVSWSpifOo2lpRkr6BO1Stimqdda2nDBxX98U0Q6qWgqFK72tmIw96Cs/Bthi4vCRNvAhQg3PudCjOZi2Lxlo19/l2M1tBgWPTc6YIW0ZxkYYYFSl/1HLWHkKhO4DG/uBDhOuKTIEL1a/kXrwM8puhZo4nC1JwjX/LMVuh/Zdxy/9dznI5svuHeyjexNsnJREdaYP1aFthGkp4vRs5JBkiuit6df6zUzMyUfSHObSuWESbfaoTRVbEQfrFGLVaJz5S3lwA1VcuhPqX1KcejXEwmkEibwIGb/xo3E4KlRW8Dxo4dQLc3Jz/f1D+satJ6yghe/5M1i1lC4/uZeUy0ns+zC82vFjxPJIcQ1O0bwlK0rsHXrFlc4aCl55u+1+AAMrFotwWvM1Qj1KZ50tFWzEA7JCq2Q4Ivsnib6RDzZ6Ddd7T9HwmZqHGNCEPoT/tl5IAeEzM8v4PDJSTzzOS+Q//QbWoFdRFaRxQ9pgggqdZKtYgQELTaVIp5Af98Q8rkcZmatwEI/zZJpoVDUJiNdV5uVVonmnUTEVMoi3VYLibhxqfm1uLhoOTJpvtwU+ncW4pNK4ZjiUF5GE2qhVl3Cwf2PY3F+Dj09fVgqMQ01GDK4+MVvEk5BtqACE1fM7vgdnzcqXyVNxVILCq4/HeItv3clRkZHMTBgfGdqnZCqiIADqTYtBQUeOmvW68voJLb2hpCZ0P19PT/a57ld8+tAlSdK3UX3Xpr0l6KqSAodw97RUKV+beaq8zh84iyuu/4ZGBgYtjRZvpbmjxvUKlwKlEgcbDWNeN6OUGelK5lSmtOpRzNflZnkBogbdTdL6pB3bfYwXCNPi2FcQoF7mi/9Lcns8tuKU6x4kkynkE5lkMrkrPASMpBsoV6v4MD+fSgvzuk69NLcoMFFL3o9QwhEZEUQNJBZ6lR3WW+zxfk1X8laa4i/fdUN4hytW7+28wKMHK3CxEXgziMXy/vgtnwwAzNPFKfgCAZ4U2vafG4aRH/M3G65ue6IbDlw0XUQekHDpc/9ksmWfzWG/1K5gj37DiIKElg5tgpr127A4OCgu58VIDzEZ9fjolJ7LMUJ4gxyMvocfV2rEcqSNeqmpboPImcdgAYpPUSamnUJiQwOXscHlBZcJZUedTnWvCchUJLOs7KGYrgYiiFTffLEMQVVrXpN6FdwwR/cqJoT1Z67k0TsA0dPd0vryjWJUHVN6PKU5JaXXougXcO2rVtdac6iXtYTzX4bX56woZTItaeI3OXyyi6nyQS63BfL0DpfawFXF9p8otC6Wu/Nbzfy9puik686dWaQQ2GTBksTWa3VMTE5g0qlhgVHMS3ke9DXP4DhoSGlfUYOIJCQknWoN+rIZXNiYLLa1aw1kS8URKy3ANN8IHlP/N12ZCkZW1pUCGAC7Kyer29TuD4KpzVUoElkLhGXcJlqiQoci6NeqwjQaNSbItrVKmVMkgR//gteHSkBpyaJdchqSlyYrUyh6vfEWM35GhzJP7YUyd34nCuwsghs3bpVHQR6yEZTjD4+VCJpEaLHpgleqCYcg3YZL8tdL3RLfTZ2Xx9oeYH5mq58iRTPAx5duNGbbtsQXdFbvODIb8twaG+z+VkFLgpkmMIQSkyojivz17bFrzfrmJmZxfT0tEjgpMSsWr1aqQwXP0PBtppIZjLa2HH6Sq4tTXQU6X3FmVavUoBK3Syc0KhUyoAKx1zhc/B3adKb9YbRaRy8SBK+8OxcQZrMtaMZr9Zq6CkWEUQBZmYnEGz/3Vcqx+EuY7jeFuUjJXqo/ITrYVER3tFYZHLZQQDgwrEc/uSZV8rnjowM63cogHqdddKGcjcJV5zgCG0KRyprQVHYYOTpfG1HsBLPsnzT0hvvm01QTjTOny4XrBduJ27oFCh8T47Vn31aJdMp8ME0Pc3WlnQajUYod6HiAIvl4mzxO4sFBjHy6+ix49izew82b9sqZgbf0PjEMcGrPYVep5mEK7kmZiVJjGMaxPfiz9LppKwHyW0sJPAzJAlmMxmhZPyZZeo09QnlvLQUbLFhlMzfZdkxESRRri4i2P68V4jayg/qwblzGYmJLEdz3MVuzX+Y6WGFgzsm3W7i7970+6LAbtiw0VVTrAjuuT7aJMtKgR7BUiRKaK5OaqxXNa+JxrxQeuZyU/8Zn654c+XTmyf64K5/dnixAyi8b7NQwmu0gRmW41r0SuSIgZFxlRgZ8ze4vPSxaYuWCS86VubMzBz27z+IK570JLtWKq51YqtModAjM8581mDZBGJJgy/LlSVZLU+WZ6DH+/q4gxuFJAGiWvKzDo2jD+YXhcvNQVdSyOdlHcSh2vbclxm2rBezfJcPRqaiAhsXOT4xkOmmMC185FXPQrO+hJ07L3DQIfFiEy4XizeKBZbndfyiQ6oyqZS0iFxb72tN84zyQwK6Uip1QXRtrU/bfMDkg7Ouj+4iTd786rvCRxY5iKBZZLs8NZPPZzBHocUTyjsJIugzrrYsLXepi6FbKbd2AaqVGnbvO4Drr78B1RohxhCBCgkpFAsDpu3tyNYkYcgYUS9qsHhsrmnNWyoJ2OHJ9KfcLHwmw/u5powZLP+lkHldYtYsagS/8+d/GR08OSMdpW+ieZZm+OYmn3g74prw207QY8X3N//+1RgpxDA2PoahoVGpGyNBmiQrAIRqWvKRnzZG2Das2ZHVqRRM5K0obULkC3iozufZy4O5bnpkSM9ysGP555ZrtH7H6Z9v2zB/fq7v5u8IWWIQRGy80ZQVD0l7SRsZUBvVce5Rvt0AACAASURBVJ+kzxR4BDyyey92Xnw58jlWdyI0XarHQKhY7FNflFwSsXgR3QKlRhScXbPLkfJKRMXLptMq5zFr4Lp0SjxtA38y2Zyux3hE6/Hhv3t/9NXbD7o2CiARTxnMGCfDwFWGhG+6PE3+MjCOkjNpT9qyAq95/tWYnJzCBRfs1NIRIvMEaj4wheuDB2lb2Fa0Z2VCa4uUTw6NOsJVoub4AGt5arRcO+1xzPH+prTHC/Ycy6Mow2izhBKNvdEVrv8dBUW0ZDH24iS1+ZSzq9vBqES6vwvSrOkMwnYXy3Vcc91TUK2WxNW2jUgYMoVEusdhyQZu1BtVaR5JbRRwoJ4ti6TlltRaY8wSghuHjxzCyMgIEklWh5iBEDWUzhsa1nJdg9/79ueiv/qnnyH03en0u/IjrEYAqXQM1bp1FJhZtZ4hARmCJUNk0MSn/uqFmDg1hQsu3NnlDIkr5CggjvBNVEV+goxBlQId6WtZIYE72gdP9D+eWvNErfWbpZvmsLbpUq4n8K2kEYIlfWpl373Gd69t2YDfMN6ke39sjVu/HuCZ8CxQa7baePixx3H905+OVJrr6ciGDlmKx9OuWY314YKUhc/BlIgpZLlUElqmNhP1DJkVYYObqk31Kk6cOImxsZWyLMQxtdk8IhvFkCT/6vv/9dHon28/hb3H2UOrBgeXWFv5Kx4L0KJd74AKXXK4pUrkHcfxN6+5AT2FHPL5IsZXjcuMMQBg7XK51tSrS9rxhWxObEj17Wr3eX6VtTF6HrJniDzR5PLnvjNuudYZsvTrAvbCXc7U8KbRKLbc7VavXf5l9zXNpqXh330VpnvfcwEXtuLc+8ADeNqzn6kuQW+dvILQ9THVYr6bTOaQK/Zbg1errjUnYkWesyc+KHIWeY7tNGyxsRbNudk5EfiowWKfOtYMGSZMKoOvfP7m6EQphy/f+nAnWrQw3UB0htwG6Fg1xptJFbjVcmhoyxtecCUu3LYOfLHNm84TdEfnTmjMp01ajHbLismOikKap9ISl9tQu3xqIA12dWFvfhVoeO2xhKkTpC03p0ZmZ4pjLsT6WrsBmTd7pv2WilFo9G0+wFq+oejnaLVk1eIJuRwxRlzXhAVABlXyfR7YtQtPvvY69Pf3IEbqilAuM7ctxRvEiJl+seGcbMoCcvkevQ+jafZjLZUX7XqOEy4cgv42ndIzsKOez8H0RzmwXA0trNXPg89++q3RyrGNuOmzdzrfR3/LJNvRJ1203GUvm18kTCmCNR+4HeGarSN45e9eh+n5Rey84GL09BSkuWQXWMe3Q5/ESYJQFVY+mO9qEZ1ZNoqN0VI98OAF2rEArhvOymce9DDR+iDLVSgFyxka/uu0WPO33cJIVyu7Mzm6m4ob3MqiipZjpNo09C7iTjnI1IQc4aFHHsEll12CYk8OYdsmDSTYMachJhX5xXS+X+lWPMloO41Eml2CeQSxtJiSdfKp60blkfAcKZ19VxSuOurn53TNbC7b6WAIkJBVDD79yZuilSOj+JcfH8b+o1OOUEY6nMN+HfWl44OiLuDgUxsKuyfewEff8hJkyE5oA+efv1PmaHp6EhW2SDrY0IQXF7NfuZjgSRLJu0ERTY/HcLm4HaE6bbSo27Dt3xQM2e51uKvSHUt7lrthM8nn8qH5M2o6SW3Gi3Ik92W/6Neh44NdP5SEx+qXBq808OADj+CKyy9DLFFH1JxzFFgyOvjeS5ibn8fA0EoUewaEUadSBSRTecRTRcRSBfnSSm1JG1wIlY8lVBa1+/gon03Y0mhOLlDKQ7NdQ/D5z70zIuXl8FwM/377Y6R3uZTIqkTRstFBZlrONW9cZJbp4mETH33D72B4YBBnzkxgw/qN2LRpE0qlBQmY1RXeuCNcNmcR0uPEGxcJ+MiQloDXtADFlfccAKENtazk5zXVm2TTeAZORvnUu8rCWITr5cTr/Obo2qJa5t1+dIPPqb0W2zo46qxD12wTMipuo9lu4r57H8Q1V12LIFlBo3bWmrXVPWHMSUGeehNG43FNCygUhxBPFhBPMl0qIEiYf2dNmPez7MNiIlvLlqwsr804xXfZczALQY/g37/0/ujs3CzGV63DOz/9E7TcOB5vetgC6X2wvrvkSsV7jwjwScM2bn7VM7BufFTBwd49B3HJJZdg3bp1OHv2LCqEwxRtW5hOXy0hsP5Jv9JiVSQ8h2clLNsX9OmLqR1us6mcKAjLl/RcbuzYCl7YRrfxjEbTVm9efUTu677dAMl+WxGsS4WWa+xy889r+MKHWJ3uHe+9935cffU1GFkxALYU+xFGwuSdK1P3tCPw6ZqKC9JoRSlEEQnrxI2bypO5FuZiDIvwpHTen8UICj7O4SexlDZLgsHfd7/+kWj/6ZMYHx7Cl247jj1Hpzo+RSaPzdNy1o4d6Adtiepq5W29ICI8+9L1+L1nXSU2JO3+3r17cemllwpvJetvZnbaWYWYmrhVrXILQuYGw35uGFVGXC7p0yL+nL64Q3xz+aUJxAoRhpEvazuJjDaz3K96VqWn9DhP3YnFfKDli8ACGahZywaQLA+0+BIiIzgivQdG7rnnXjz1addjbOUYYlma94TGIPFZWxr3tIyG6+g9aRYKckXkC3kkUnnX+xTDQmkRZ86excLCrFnTtuWz8vl6P3N1JKtnM0ytYmZxv/f1D0YnpubUpHx6MYav/ehxPagvjWnhPEOQQibfN0qiFYRIJNOKfjX3ImyhEKvjIze9VNUh0kwYeT7y8KM4//zzsXnzZj3AwUN75Zv4YNJcji1wmqvyVaMu4dIcaTe6tgnrPjSWoQffmdQnU0YIp0bL50i4XW31qYw3rWbGfYDXbaE516w7uolDn8gu8ZbMPud4Zq5G2+IG9dYhAirVCu655x5c/4ynY+eFF2oQC5+vk3WcswmNC95xL9JkC9iWuwO/QalIM3OzapEpl22kBFVM1lANdsSWyfJIIPjfr70/ml+q4tTsPDasWYc3ffqOjnCNrWipAp9MjVFZYPOaAezcsQPbz9uAWz75H1gx2ovX/P7TkE3FUC7VZFrT6ZzmRTDUZ68pWxN37NiBQjGHAwf2yzQp8SY3yY01oKkV66/eEGtQezJsKyDz8B9pKIcPHcGhQ0dw9NgxlduuuupKrF09rqCF+Cs3j0YykLSuQIqL1aURWTDmYE43XW65cDtq7KJvXudcAXd5VsKFljEm+S58h1/96le44ZnPUBEhzplQ2nHehzyxJt0dIGZ+ffmzuu3kGKl87tLiPM6emcRcqaJqELsiFFxpqk0K2Tznb1G4X3l31IxiOHDiDMZWDOPLtx7AniNTUutUMsC60V485bpLce1F5yMb53xHmkBruWADcTqbkuuYmJoS7tlb6EVPoYBUOq2RCIlkVkA3AXXWQM/bvk0shwP796LJAWGctUEwQw3EVs/MZmwWpK9fcrFKSwtaIHKEjp84gX37DuKO2+5ET28fLr1kJ+LtJlauHsOmzZu0qTRPg01W7BdS7mrm2gvZAjuL/I1GYwv6xC+vUfx3n5J4rVoeYBkUa0Ej3+PBB3bhhhuejiuuvdoVZbqdeL92k2UQqv2bFS4sVXQBbKuJ2akzmJ6ZVFGgEcVRbxmGvLRUsljFtdzmC33a5MF3vvLuiJPfjs/MKj87ORvDV3/0ILLxGN78it/CRTs2qfdn4uRprN6wRfRLmuC9j+9SJ3krTOKXd/1CZcCFxUUc2HsAr3jZy9WZRhPBIWJkOxBmSybi2LN3H87btk1Fht27H9XIAj7sxJmzqoyQj0VWA3egLb7xsirVJWkE2zsOHTqMYydPYW1xCFG9qsbpRrWKRgJYt20ThoaHUGs1JVzyi/ni3Nm+/so/GwpmVBV/Dx+FPlHIHo6k2yBa1HVb54rJR8vVag27HnwIT3/GM3HFNU8WPCg2yzJi4BOjfH8lu7frxgBQa9QxffoYSgtzaJBRGhJnCCXcKGa57fzcrA2CITrXDFHs7bcJct/60s3UZsyXazg9s4Btm7bgE1/5MV7wjCuRj1XVS1ro68emHRcjiidRr8yhVpoWmlKuR8jn+9yIO0dRbbUxPz2jZyXXltrLB2ZZjLSRXKGA++67X1E02RuPPvIgFifP4rvf+g4ufdKVWDE2rs/5sN4HKqwPc3RRvdHC8ePHcWTfQQynsujLs8WSvUllzC8tYmjtKM7fsVUWZrFcFR87xdGDyVQnhbCufqONdiNkC+TSKeK+TzSLnrZjsQjZKOf6w27RgRpM4T70yMN4+tOegSuvuVp14N9kFcx3L0fNmO/bZCFq4/SZ48qJbaRSiKpGB4bIZQoIE1nUHHGuUq6hXCnLlTFmoUtU0/c3v/guX0XE3hOTippXbdyJ3Y89gFw8wujYWvSu3IAUZz9FTTTrC2jXltAKEsgWBhUFSqOoOfU6ij19aNXqWJif10JQo7lgyuViceSKBfT19eKB+x7EwNAgxkZHcdu3vykh1dshRtas0kPy4WzhLX1imjE7O4elSgUTExM4su8A+pFCf46d7m1U6lX1xuYGcrjimisUMbZiccwvllEikzDmmIjkHblZEn4DeXYjsWP6MFZ+yDI0k06/7SBS189kJUDmmDZNx3OmVbsNgHK5ir379uGaq6/FVddd64r8Li53LS+/JmyxUuqYmT2Lec7LrNfdcE9oXbnxyK9WR2Isg6Umo27bGKTzkG7D9hXSbRinKCf+1hf+2nqFogBHpmYRhgEuu+wq1JpttOp1TUDjWFo+dbO6iKWFKeVjAyMczROhNDeD5vw82tk8hsZXCW2pl5aEexriExPgnsykBZnx79TM3t4B7Nr1oBj7e++/D5kgwoatm9FkWp+yGipRGmbTjKa5mATTZ+fnMTM9g8P7D2FxehYjff3oydA8BSgOD6IwOoih0eEun1Usw4baNX0hnNxhBmikqXLhatWqgjHOgBalpc58NYZiT9GE6xA0HzF7zhN98HJTbmkKp93VsHv3HlzzlKfgmmuu6RT5zQqFnTHBNJmMNRrVRUyeOY7y4oKCI2IJFKZvDyE8KUvBHJbfEynML9VYFHWBeyDOMiFhC+hamJqcRPDtL1qXH83JbLmOU9OLuJBR7dAqzaZi7hnGDRWZO3tMTcbJbEFQcCpJQhwDoQYKhX65FvaJEvGamZhyILojgGWMrUeB0c/1cvBzJot779+FdatWYf8v70Ihn8OazRsxx0Atk1IVBCmaTtMG+v75xUVUyuxqT8tKsH9GMKLLc1nFYpuG9e3GbEYTgXe1lqq0ro/ST1szN2dUEu+mWSaQ0hQ6VVqYFz5r44KNxiK+kpvURgEzNqAZNBpOt1uBdd9HH3sc1z31qXjyk+lzO0Qv+Uj+ndy0ytIcJk+fQLW6KH53k0WSJsn7ZFOSvmpIFAsMCt5iFmSSgltpkhBhJVdqqjjXgcGP5FiJ2fHNf7FGMI3yDAPsPTmJbVs3o39oFaIgjvrCAtJ9vRJYPGgJzFAaodJgVlFoNmM7nNQaLiyF3Wq0MDs13WFAk1wm8jY1OMEZy2lpMCm19/7qAawZHMCpvXsxso4T2xqkIyKWylgwwiqHgxUJnfgitpkkTmo1890FLLoN5FxMgyO7RQXLGQ0dEuOSlB5XeaFWW2pjuTsjeRLqOW5vbm5GP+dQElJX89mcKjJiNTLPThqZrlKrYvfj+3DtU67F1ddcw+FMDg82hGx+ZgIzE2fUokJNVn8PzXAUiO9MFsw5QnUTbLVF4glUqk2A9CNCrK226Lj9w6PdGdWsBbNyRuGqYC06TIADpyawdv1GbNywFW2mEEQWHZZKDWCnm3BZ9qLG0+jt7Te/26yhVisjrDVEDR0eXYG9j+8RLKnPtw37ZARLn8bFKHJCTC6L0mIZpycmUDl6DGs2rsfi4oxeIl3oRZDKoCnGhJ/h6HqZPA7qWCEUrwB117qpblyVYq3tXjveIQF8Ht8uaiOZ3Owt109rBQWrSrEUqTmTRJTccOuwXcfc7AxmZ6fR19urLkc/zY4bmJp7+PAxXHX1VRJuFBi3eebsMXNj6vUx00sqkjfzUAspe+9c2tQBMwwBU9kyHsMPf3gH1m7chPFVaxTcNVshCn0DHfoOPyn//81/eWvEtMBrxHypghMzJTz7Wb+l7jWNi3YDNTybkeY4mUkinbIxAkxVGs0qmuUS2osV9K/fpAapvbv3iF7jUweLmq13lSMDucv7+wf1/Z7778O6sTUIykvYs/8hjK7bjFTvoCoivvLj5CRhCfJ04wo0Es+xHXwBX9MAHCfYpx0eyvTVFJ9HL09tuqU7K+WpLqwWDb+pBIFIo3lfrs3kmTMcsY5igZkB90MME5MTuPa6a7Bz5zZMnT2OWpl9s37crnG2WdNlPup7fzS7QGbVI2dPqC3HOA8jwkf/5uNIpnO45tqnYMt55yMv1wRkclmHt9scseC/PvfmSFV8B6k1WxHueugx/P4LXyK+LbvD+SCznP+QTGP16rXadQl1dzNftKJ1q15FbWZGbSljm7YreGLktm/Po520wUAEQ1E4foeLTIQpl88p79z92B70sojdm1c+J0L8slKar7VbwYBgipkl0VAcFUXENd/muWyEjwf4fa7pUyDTYqsYqStedVOruxpIYa0kFnTan+05bF4yf07OFznHQdhW8/PExBnFB9c/5ToU8zarmo/ZaFpXQE4IkrV0dm7C6MW5ZlpF8+OOrOhBjlgMJ06ewQc/+BHNCxsaWYHXv+ktij0azRB5Np4x3FCfcYTgP/7xzXpUmlz+WIXmvYewfst2jPT348DBw9KQy654skwQc82+oRUqDRqDnuMLaoimZxGL2siOb0CChyjEjPz16MMPqNWh07SdMNCbIb1FxAl1l7MT7pe/vAcbNm1SSO99pC/h+QqO95Uap6eeHYvkrRuCwZu1cHQrPsYi8f/7EqJPRfzPbbJbl9WhAMmPTHQjkjT5TZzh7qR0r/26ju8NFvegjVw6iXy2hWaNuWoLmYwbdURzy1JdJ8c1IXeY252GvHNRM6aTd/70LvzdJz8j4W2/4EK84+b3qomP8Gg2Y/mtbcoAwb9/5k1OuJaYs8Q2PbeAh/YcwqXbt2KhHql01T+4Ev/38+9jxchKjK0/D/EgrcixVZvH0vxZpEoNpIdWozC21pj5Lig4cng/pqcmdIKIaY2ZU/lfzk526BXH+iwuLOHw8eMYGVnhGJR2/IpnGcp8uglxHYTHjTDwJns5mc5rpc8GTE3cizu1tAmxbn8otiABzj2rousuDuz9szYGBehmdvjZVJ4HaSXFNtKZvEYg9fcNo16dRKs+a5Qj+/WOpvp5HF04wz/nE8CUII6//btP466771d6+Ozn/jb+5BWvVOBrU+2t48BKnKBw36gJcmEH/LaW/Xt2H8TGNWtw4YWXotA3iPnZWey672dYsXIMW3dchky6iPLCBA7tuw+57ADG+sfRt+UicXqtucpSAx7S8OB9dyNOrpDj+fA7fa6OmnE9OkX2GQUBfvqzu3DxZZcr9fGC8EwMn6f6n1sB3gKp5ZrZiYZdXqmKjINqrH5qYvAm2goMFlVbIOX1yBMTltNeu/hzJwZww0qNueEHkLLQQmw7jkwuj6HBQZTrVcSjEpq1WZc7n0vG0939XI/fUECgaX/t629CtUpX2MZ1T3s6Xvryl+tMKP5erdFQFuKnCwVf/4c36LUpXJksle9CHDo1hU1bz8PI8CjSuQJ6BwaRipPUFaFaW8TxA48gm4ihf8UmJHODqv4Ucz0a7mE5HxecM/qr2PXAPZrA5isXFlg588yyXTyOniJpJik8sOsRDA6v6IzD96R240tZ0dvCYMe2kCl29BbHenyif9VMLKe1DF7oIkQJdYgTQxjXwNQpF1rlyIRtDeF2gXPcgxMGzbVr7O0Ef4qAk7bQyQzbSQrKQ+MRjwaYVm7rvzoQaOcnnlprEb+n+0zNzOFTn/4X9PYNYnJiApu2bcefvOzlnQYCOlaS61QPZo78b59+gzTXgoouC35msYTN2y9BNstjYQjAk4zdxOLcWcTQQKFvDPneFeDZBlxTTVlJsaXQIDkLQCKcOrIfU8zp2k5THAfI+1vOgOTn8wVrS6xVG3hs736sWrOu033gCWjLYFg3YceqPN6P+vfgGikgcX6QG8RXfTRYzD2fX0uNmu+0itiIJPP1ftxg12BaccB3OnY7Eq3ebFCppwslk2zKTulUFn6nzw0Zn4RltBqz2lBesB1b4SpTy+FJXwI8PTmDNjJsA1Ne/Nhjj+OGZz5LWY02nhusQsurkunXPvlaPbknZ1NDWACu1ptYt+V8FPuGNMm8Xivj7v/7KebnprB9xw6s2bgdxYFx8AXIv+WD0wd73JYPVy4tYveuX6G3bwBziyRac8QdI1L7zuCHs5Ysz7N+VP7stjt+hksuvVz5ogEmHIVnpsenQNREnYe0bFyNN2kqCngSmaOqGnRIgfvJriZwC4is8/CJvUjeWpwjANfD5FOmznBxZ04NX7aUT2iczjmyYCuTIaLXRNRaQipJFkV3/qWE60bwWKuSoWxyQSywRhGmSzWEETtCjMZaXqwglc1i1ao1+igbC7zbYQQf/OunXhdxp1pfj43jY1sDnXMdCWy74CIdWrF/zx7cdtvt2LJpAzZv2Y7x1ZvRjJoYGlmP/oERaS3RJg/FtRs1nDhyEHMzUxgYGMDk3LwwU+/fDNExAUu46YSbeprC3j37EMVS6OnjSPjuCKLlEa4/tMo3mynYcoGQpsI5cr1+rsFgJkjfpqmBmD6lUm65nBbbnWul1EqtIxSEoUky1Y7Evly4SgndsTH2nkYYYFrHAaHV8gKymRgyWY45CgVuLP9yLJyuuV5mqjgOa7Yc6nAsmvtENo0ETyqq19VHzOmwtKJ+I8p6fvXvX6ujZwhONzTyrqkEee22y1HsH9ZBi4sLUzhw4BASyTx2XHAZKrUKZqYmEdaX0De0GgNDo+rGsxEANpCkPDelUbezCwvIZbKYWeBQLMsLVUiW3zPGhE61omnO51UDZhPxPffuwvYLLrBTTRy8aICT29HkR4mw5ykxNtRSfCcHPviN5lsdfRTsN4EKG+56Ppiy/lc3DYccY47Xd5+z+c/eLHd51f6kFPEEHZxoRRMOBW8hk0pgeuYsVo+tIOtUmyOZYAdl97wGmXpvO57Qt8QNxEHeUaoPuUI/0qkcEnSV7pwhsJ+ak+fTPPTSql7S+K/+/euiVK4Ho2u3KXlv1BoYWbVeH6Z5TjimXRBY/sQXnJqeQF9vj5sbxY50G7ZlN2P1qISl+VljPnC2w/QCSP46PTOtx+8K1ygx2hQOsert6ZWQ7rjz59h63g4EIqgzv+yO75NwHEvTFtGzLLpzlj1DUGxBD+xbmN0BQCzNcXO2XAqkpfd/duCGKLK+q93P+hAzk2OJSBcyDjWtnQnXNkQ2lRQxsJBLgu+lwMsockilz+2UWB6pL8/teb25uQUcPnwYq9adh7G1W9DTO4hUiiwXg3EJW9qGtf4romd61S9/4vXRiq3nI5HIK6pjlUWtIJW6RgDoFCoOvmzzcKM6cmK22/ANegMCGfQt9L0UFAvNlblpla6IYvEomaDOMCCOx44eQIXXJIHakb6lvQIzLPft6SmqsH7sxGmcmZjCqjVrXM+SI2LTZzsSmZliq/6YkE1QVvN0vKkO2c/G/fnPLE85OhagMyfKLCPHMYlD7doXdLiWEz43P9+Ri0/r4sceklXCAxg5PJtnKK1YOdIZgeSjbzbHxROOmit34BvNXYDGokWbaFcZp06dVA+xmr2jAPFMP1as3YxVqzfrTCYxQlkN0sxmP3nWGgqC7/zrR6P88LhmHBWLPXpQcp3YakiTxLlH3tyaBbNo0s8O5qg6aq2GY8USaCzOqTrk5xSngyRSnEIXAQvVJew9cUQVH5XmNPfBqikKrkjNyWdVCmRN8ud3/QqXX36lDfrQZFULMCgMzy+y/NaFHX4iTydyda353YpbR2spKA83MvjwFsBCWD/Px/hixDYJj7IU6IeNWiBGoRL8NyYnW2OqpQVNERgfHztnWo+iWXfWHwVrYyP8gBd7Tn8e4NJiCSdOntS16ars7Swby6TtfNx4pg/9I+vFN89wyLdC/nPhyuC2H/5bRJw3X2Q3WoizZycdMTzUEGkS1bgIFCJ3K2uNLH+RVuqHTZNpQQ1tc+T8XT/HtvO2I5ctIMuNQVPhpqtz3+86sBstapejslg1xa7v76MwPhbHXb+6T1h2b1+/sxTdoZ8e7vNsCUOa7HwDLrQCGuOSdhbHarx+qUw7O2cYOX+uxm9+TtGNMSRtWJEtMDcCzV5VZyOQ0mr3mmU5sF2XXzW2KIsOXRjUT+JRj0HSpp53K1Lmq0mtOXDwEKpLSxgdXWHjiJQlmCZbI1gSuQIPrqJZziEK0ugdWo+RFStRKPa5Ax/dO99++39ExIz5oJzq3d87pAiMtJZCgR+2vJXaLJSHuRTYzkg+1ZL4SQqE0hkc3bcb85OTWLNmHYYHR5F0A6+lFS4GPDZ1BmfmZ7UA1Fz+G30wtZ8Cpu/VOKBEHNPT8zh27BS2nbdD7kEpjitg+2jZzLAhQ/7L/0zYhIMrO4L0vUeuK74DUWpD2KQ4/ucn1Sr/V5Rscyq8gHk93pe12XJ5Tr2ymTQ7BZYNanEdi517KNWhW3LDXpbVco8cOaLDL0aGhxXrEG+3KnW3GuWRmGQmh0K+1wWjVvM+OzGHgRWrse2Cy9HX02co4T2/+l5EVsKx4ydQKPbI52peAzHfXI9elCdv0Lf2FHskTHZ385i3hblppNI5jI4MY/L4KTS444YG1aeSQEJlMl/p8AhRI2rhwf2PK1ezaNbGDXCHCs1JsVJUEIxG6PaXd92LKy6/Si/g/amZZwcj+omrHXDZRu8qFVgGxnt4UubRFRYsJ7Q0iD/r/N2fgOb8qyJmFzCRQcFrzc3PLru/ggAAIABJREFUYKk0i9Xjo3pW+XBtnG5HIwkOZmq5Zaj9LQRxOwyTm4Zs0aNHj2J2ZkbnFRFZ0nFvbnC5z7t9KuZNN3nQFC6j41SSGsw4xI7RmZgtYdsFV2H9xi0IfvqT/4h2P/4YVq9ZqzPouHttJA7HyfbKB/OXaNd1OKBjYnBw1uzUpDjIuUQKpYkZDA0MdNAfP9p3OQBgfqeFr3//O9i0eaOrYNh4Wz6cZzIwnCfbga2Kjzy6B4MDI+jrH3Qmx+G3rLE602vAvfPFjvzmBetrt7YhDFnSoBPXKurJ6SYEX9pz5xe6M+j5b/bsbSzOTmJubgLjq8ZEC1oe2Yp7tOyod4tPLCibmp3DihUFHUXOya/Hjh/DwUOHMTo6it6eHm0e0op8XOHxdD4r51hpgqxGRXEgNZmkRTueNmEnsBlebyOUJmdmECSyCL7++fdEHMG+cs1mjK1ar74Ucl4505+NQuyx1bBsjTHi/EM3PbxeweLsDFYMj6AnkbETpt285nO8moWXyhxFYYkFeO5LX4Z3vuMt6hAXwZ3+F5YSMWKmBvf0FvSgPOzwyJET2on0611UyU9a92mQm2LufKefq7F8croN2zZ15p/5ngySRFZwzVZ+cdWzpAOTQ7WlUlNLi9NYOTqCQj5j2u46EK3Ga5vDa7BVswxF++4P78Dddz+Aj9zyOkxNT2Lf3r2yTr19Zlo5gI2j68lKoYA6DXbuXbhuXTDHxiczFmJgxX5epaFq37QAlUohyPLv/vpFUakWYfV5F2nsnI4hjccwSE4ObGIKaZP0cfTL6vHhGLp2iKF+JtRpHUWz3Ox1nB8fjprSbopDnMrnRNt53p++Gju2b8Hzf/vpehBjRdqsJ0bMFHCxyK4FnuUTx91334ftO3fKBFmC3q3MWGoDQZ8dGo0QKhOgNprzu8p53XytLhZsAZHH1el+6JYYNHHYWK26iNL8FFauHBFA0PGp6jrstDwaNKoGLyIZEVpBGydOz+KTn/o8FkuLGBwYwkteeI1mJtON6Zxg8q3ZoxwDFubmbDgoWzTl9hwJwQWI84x5AlaasupgoExIdWUNlyenKOMQS9LOHpZb+shNvxedd+l16B8dw749+3QE2tEjR7CwsISt23dgYHBYlYZimvMu8hjs6UdagRIRlq4YrRtx2Q98+N6o4czJExhZOYZ4Oid/84I/fx0WZkt44xtfgeFBzoOgcM0kUWv5kplMSvejPz5y+DjiqSyGh0dd173ddzlAYSaXARePYHU1WH8MuSvvdQKbTnXHepE8ZCgNceNwORvq7JkTWDHSp/NwOTGGhAav4b6Wa6ObzBw3eARAixScCN+97Q5841s/VEtlNhPH8OAw3vTGF4v1SQ3XmcANbiIDQrRpHN+M0/uMPGBf/Deef3Tq9Gk0iRnks4J0h0ZGFQel06a9VBSRIFyeH3zz6x+Phletx5mTp7Rc2XQSX/rCl7B27Tpceunl4JTwzRu2okedA8ZW+E1fFK49ibwTKxGoLc3h5z+9E2s2bMV2jjCKqHUhXvyXb8HZ09PI5GL467e8FmmejcuxO9JAlsmskM+UiFaEk7+PHD2B0RVjRrBLpmXyvLXwEKKHNm1mRld7LfvpTqDx5pM/JqfZLFJT7S6sM09NntZpoiOjgx1GiAnVEDrvW71p5jtxk9Q4aysWx/ETp/GuD34KYcsg1mw6hcGBAXz4Q28UT1rAB88jKFn/kxq5NW7fToBRy8oyUEb+lmPzS0uYmyXt1w6SLvb2iJyXz/WKd002i1lAd8T5F//pAxFz1rNnp3HFFZfjJ7ffpl1D9kUmSElT1W3vGAkdGTrfpS53tWCylbOFiCzIyhKWJk/j9NFDaCbyuPpZv+PGGNghha9427vEDuRqXbhzM17yB7+tUXsEJhhUkBhO08ygyqbJJoQ1U3PZq6Qh1X4QqZu/yMdRpcnNjrDJag5udCiQByCkqRylELfpdqwgcbdPT51BPN7G+PhKd0aPHVbh0yLvV7WHdZybzV8mIcGDIAxA9+zbh4//w9dVClXuzkOVB3rxzre/WvEF72/zH+3EFJpQ+uaFuRlZBp2P64oZPuQ3q8gzI1qoN9nGkxfgo9abZEbvzkEognY9h+pD73ldxItf9aQn48CBA3rZiy6+GKkwQDHtiFwqR51rdulfNAa2ZsemVOenEOdIQJ5Z16jLvMdSeay96MmaYkoHL78UAH9+8y3YvXevMzltvOwPfxc7tm+ynNoFVSSAc3cyyODP9x88ikQiJy1jBYQ/Y4DV8bXLqkIetfKEuu6UmbYKI57KqxJlLMDszIRGGaxeNSZBG4fbGqS9ufeaK+qsw5c5Q5pDxJSJRhGOnziFvr5+ZAsFvOEtH0bDzY1MpjMY7C1IuFQO46W7yTgc6En6Ljdcg90PFU0/50ZkWUE+mNNuOJRb5/4lELYthdTQz5z1QdGi8GgaNb3FHI/q5re+Mrr++qcaOH3oMK580lVAM8Rwpsd6PL05O2d0fQvVyrxYfj++7Xb86r4HdajgZZs3Yf3YKMbGV6NnYBgD4+vVKW6zRzwJLMBfffQTuPu++115ylzBe972F+DBO9Q8Etf5kNydjCopyPnFEg4dOq42FC484U5G8fQ1Hic2SNATD2yulI+W+TtqHWGJLGOp1vzcpGYhr141LsjTJqC7QybF+DB/p5O3NbbQzCZhR54qcmDfbhQKWUxOTaspfOXqNVi7lodo5fD/Xvse1Oo8M5gDv1IY6CniHW97tdW7SSrUSAbLsdVsLetBrW6qTKp7xY2KlMkYed9X3hIJ6170AJOdY2A5tT8mT3L78Xe/IFL6bbf9RCnBti3bcPXOy5COudFzHkxXrYrMvxDlyhz27XscP/jBDzAzXxadc7C3B5tWrcUN19+AdTyQKZ0hhKMN0nHF+kMM7//MZ/Djn/+iU3ukW/jWFz+FBx9/VIINknEtNmugFC5NGVtIbrvtDlz15GtQrzfRFJhgG8YPlubOJiZtrBIrpxH35eBuCqdY6FHhY7E0i3q9jFWrVmgD+aGhDGgsv7RyngTrThmza1LrQ0xNnsHBgwcE7Oi6xaJKlWxyY/F8aHAUr3/jLSpdKv/MJtCX78Et7329jRkkDVjHxbj8OYwUS6jGnUions4vK4l2Oxk4zoj/7kcUel61jjBQTGD15g6n7Nv/+Q/R3Xfdjf6BQfnNi7ftxNjgCOKcsuL6beT0XWms0Szj8d0P4Xvf/S4K2SzGCj3YsmYtVq5YgZ7R1cgODKnMJ5RIp2B2kSJFlhHwsS98Cd/58e1d4SaTeOlzrsOhk8dxw7OeocCAmknmIBeOU8wZVd7/wC4MD41oLmVPbz8WFlxwoSZrM/sMjLjgZI/QtHlghCjc7NykArqxsRXoLRbttBGnmZ1ZG44kJ3qs01g7l7aF+QWOK2AbiE2Y9XwqahGJgTxmhlaBh1fc8uHPolSy7ox4OoHefAEfeP+bHCfKprZy6IufocwgkZuYm4Gon01BT1rLS2RTcLopoyfuGY3SY+reNnYO+Xr7G/8oklNmJ3wqhUu3XYw0eUY698ZOu1RJzCrlKJWmceet38OK3iKGyK+KJ5RM50fHke4ftqiXeVbMGr40CoXDOhs1tBo1LC0s4HP/+S388N77O0E3g4DBZF0R37btW/GU66/XHAn6E1I1RS5rRzh2/DiGh0YxNzePM2cnMDQ8iv6BAWkTy5OitOjYPU55M1YJBUJh9/X1YGRkQEL36UU3Z3Ujf6Wty879pSYT0C8tSqhVtsu4Ide8htGDUvJ1misZBHbWXzqFv//M13HmtKtpp5LozWfxznf8hW3WJEuCPEHMiPCcqZFMZJ2JhgrxBubknZ9lA3oDrbpNjvUzvbS2oiF1fbhtBnfMzYfefaPMcjFfQD6VwQUbtik2NkoKDzG04dKRQP4Qs4f3I5ydFVmOF8rlCyiOrES6f9TNfnD0Fe52oj/Vsk6VRtOO29514BC+8oPbcHi2y/7jgl+ycdgCmaiN887fgU3beE57XmXInl4Ook5ganJaXQ/ciHzJqalpzMzM2GCUmLV9avcHQD6fRX9/HwY0G9HoJ5aFdyfOdRAmP16XTAs3B5LPWqtUceb0aUycPSNTyCNiOHhT4xjIKNE0dNa5Gzp6hpG82kUTSfz7//wEj+8+pHuyJbUnn8Z7b/5LG0TmFl9pUo6QL/0nD/AwJicFqQntqZy7r9F1WjxeQH27bhiqywhkWT17Q5mBnRYevO/tr1J/biqRwtjwCmxYMY6kWh9ddOxaDgk/EviefvwRxJT2hEjnC+ihYIvWDKZ2SB5VzinfHhliEzNbT7jAQUxpwnd/9gvcdvc9jh8M5bTPvup8ZIhO5bJIF9g914vBoWH09PYqOhYzslbD9PQsBgYNwxYJzc2y8JwmY9z70UW+qmLRvszW8vmVLne1uVA0s+zlYcddC/OzU2r24pxGf+gGy3xceG4KBn40wfSBQvCWEdp41t6P7rwXP/v5A2aWkwkJ9z3vfIMazwmQWDRuw0KTaeatHE+UNgKgH3LKe+j4c0Ph7OBIHqdacfSiLljj82KRBv1RfR96141KhRixDff2YcPoSvDgTD/7USmQO4I7rNdQOrIfsXaAdC6LXG8f4qkcqqUyyiwibNqKVLFXJ2VxxAJrssKklUr5CkwM//vTO/Hxz3zWem9IR8lk8OG3vhbzC3PI9RQwV1rQGQMUDflXg6PD8r90EzPTs3ZatNpRLD9VoVo5rZHh/J996VY7ezlo6e6r6pAOQbSSHjfP92+9A0vlBjZvXofVYyPq89H0VJ1cUhELhc+txvCwpT5aXlusRzeXmQDLfQ/twbe/+38WGNEsFzJ4+03/D6OjIxKgprRyPiOggxfTghHJ3aYw7Xp2wkuXdO+Zm3Zws6FcPl2jxVJly5Jwe99//ui7Ipaa+vv6keFAj/ISkjFrsvJAAf+cyqYRcpTf5FmwNsTLNGtEayw6K46tQW583AZcqZ+UQmXJ71xIkuz42+69F7d89GMd4TItufWrX9JAMz4UB3sQ0OfDz8xPo9pq6HAMCXeGDWkplxYYHu2jQ76XMRJMRa1Y77TXUWU8AMEDl6xxmTQZ5qsVAQnTM/M4dPQ09u09iMNHTugouysuvgAjwwVEnODGsZWMSLlWzWVn5zqYUGa11cLEdAmf/cL/mHCSCfQWsvjL171MgSfdjabPuCNTWxGU65L7zdydqRIHenpivEb2u5KnL5xo5kUQE3GCmiyNV9sUG7vdCTAP/PC/VbYm84C788zxowjanGtkfKMkT3TmYLFiBgEhsH37NYIg29OPAgvy2YKqFOzPpTnQ+RmJlHYjMWJiwjaBjlvJ2kzuevRxvP2975EuUXPZp3vrv35ZwtWp0hSSK5izk+705FnUgppaFOdm5+0AYo2nd+Q68bGMmd8Vbidec4rsit6aS9wWskQhsFG80axbLh4Ztm2RsJHeHn1sL35170NYLFVw3bVX4rxNq9FoVux+jgnpo+YOzTaIYanWwic+9a+6N013sZDBm9/4p2qmozknNswhbUaZpY5EYL+UqkIqX5pSdI4RaDQ7tCC5pERcRRu6iqXFBVeL9sfgucHhu370DVdM4WG7IWYnT2FhelJmWQm4qxVm+iy4qR0/pVn6if4RJHM9iCcNKGjWKhrn/uiDD+PA0WMyw8PDI1gxvhIjwyPqITWzk8VDB4/gbe99X6crgWfhfP9rX9FRLOcOs7YF5gY4NnkcyQyHrlggxdTBBool3elY3U6+31ihcucjUbCLiyXc8dNf4KKLLhAQohRe+C7BBJdQaBNwTqTVoE+emsTP7noQp06dwW8983qMjfYhbHAarSv+O/qrzt9jp3wb+JtPfEWCIlqXy6fx1je/2s7LFeskrRo1kThNWFW66ccb2sRYG75oftUPIVWg5F2SG0ExO22nf9J9+HhDbuKhH34jErLRamrcT2l2GmdPn9KL6awb1gqpwfksRsm7ZW9uIo1UlqiJTUZjvrhQmsfeA/tw4OBBlMo8ocqalajRzFGf/zvPx9133418Oof5ehvfuO3/rBICoLeniG9+7jPKB0VJRQxN0UaJEkWYnJ3Fl//7G9iyYTWuv+7JOvy3vFTFUmXJdjurIW4soLkTP1/ZxceCDEMslJZw+0/+Dz/40e06COrmm2/C6AiLAw6Zct37SuEYNWsGpdV0ucxkbB4/eRbf++FPlSX83vOejtrStANM/AmWjC/4/CE+8rdfs7pxPKHo/S1/+SrN3+L16FsJK1KDqcmqTrkZV5y6ahuUczq6p7r4oeAUIYNQz29bmJsVE9NvBApa1uSOf/vniNjw5NQZEc0pKpWjWk1MT8+glwXhdFoQ3aq1a9Db36cqBPFMxp8cgsVZEfsOH8QcB4ER3mPUF0SqWTLFYpf5eVu26gUe37MHpycXcOud93XsJs/Cec3znore/n7DZtMplGsGUByarOAb370Vz3zKNXjx7zzXqDl0GfGEpsZMzU9jqcJ5w562Y2ffSqNaLSwulrHr4d14bPchHD16XJ0Nx06e0Dm1N7/jJoyODihuYFM0F4cUIS4Uf9/A+7aYEF3NsdLfrof34Ps/+in+7BV/gkKKXRqLLmfluQ4xpT/v+5svytwyoi8UcrjpzX+mIwI8zzqZsLH6dDdM4ziIjXMjKXhfs+b29IdaaWwDB6O0TfF0nlDCArNyhcfcdAegqcL08Xe+NuKLLtWXUKtUxHxioLHIc+zicUxMTKJaqWJ+dkbnEuw8fweuuvIqMSNJb91z4ABqYRNDK0e1A8+eOaOTMxiveTNXq9bQbjSVwJdqVUzPMtj4b+uLBVAsZvHSF/2WKjAcA8hRCY1aC/NLdTyy7wiedNFWnDe+SlrEDvYCoT5GlywuZG2ICscZ1oMA81U7vuXHt9+FBx/ajanpeaVNrMyQ5VkoZHD0+FFkkmm87z1vw4rRYWnoxNmzGBoi2Zu5qz/pxNXA3FFtqUxS1STGJxTw9MwsvvSV/8YLXvA7GBnIIQrtfL6Y66h41y3/qEMb1U1RyOJNb3gNNmxYa9Ug1wnJP9MCUmg06by3SIeFvOsbNlNtJWM7AJp+Vm04brYW/S+DQnKlvd+X5v7TJ2+OGCm2G3U0a3VMTU1pRA8Xg0M0ieOSlcegIGgRUYkh4ujceAIDw0NYvX69Ruzk01nhtoxyKVxqlaA0IjhNO8yCmpDv6dGC/91nvqYAhuFTf38eb7jx5dJkWgL+/J4H9mD/gcN4yQufjRTzPV2ngfnFeUWDnDtJjdKZd26A2cCKUYytWaPd/PkvfwMPPbJH4AADOsNkk+jtzePw0UOiztzynrdjZGTIQHoXwPmDMbyfs/GB1ozGhSeIwHzT6rIMxtr44te+iac87WlYt7KAZEDqqmnVX73ro6hVeaJYAvlCBq+78ZU4//xtnWKMvwfNq/lcwgE8yKKtaTl8Lp2z60cbsmhfrXY6++mX/UHKlo41NaLI/G+E4F//5W+iM2dOIxUHlpbKDm4rKaLk8C02QWtXsULk+lmGhodRHBpA30C/hn8xVO/v7bP5vxxTSxDc1Vl9ea1UWhJ6k06S1Rjhbz/9dauBBsDAYBE3vvqP9IJsQ9z1yAE89uhe/NFLni0hMLYQsx6BfDmxXTtjz8bl816Mbgl4CIduhfjvb/0Iv7jrATuwjvQdca+TGB7qx76D+/T7H3zfX2NoaEDvzGfxjEnr1LMFYkSuAr0OnrBeJ8KFJMpzQo8jYeALX/0GnvPcF2B0MEBe/TpJ3PT2DwpfFpO0kMFfvOYVuPCi81T+ZKRO7SI6x89afMFOwIxoNjzPj0Il8sWtJSVxETOb9jzvi9ZSE3S46Vx9mvGFNPcDN98Y2bwKs9fUAiXXjmXPCJoLx7lSqqUOD6Gnj6U2Kw5QW0lUJzDPxaHm0m9RA/1sRZXbGg1NdWVfEa//uS98y005BUZG+vCaV/2hFmrvgVO4554H8cd//LvCYBmpas6FO2SZoRLNvDr53GljFDIDHHUHGDSGn/z8XvzgB3eq61wYsOqmCawaX4FHHntE2POHP/AuHTDJ5zO41SJ/ai8jcT6nHcJkxQhWxGgiqT18H76faqzcdO0YPvyJz+LNr38dBnptI77vQ5/EsaMntSFYGnz1K/8Il19xkfwwn1HMTOWnVr7zG4w1b17bxtvbsTN+SKnaVTIZbfIyzyHmsLNc1obOOKKfSzwRfPDdr43UOeBAc2qg8XTbMq+TUzMYGBjUgQuM0AYHhzoDr7kQWmROdOG0NXcMGqmwxFfn/7+mzgRM8rK6+re6uqqrqvfu6dl7mE0WJUgMuMRoTBRQQRQ3cIsRo3GJC4gmn1E/RFFRZI3osKkMoCCMjiIiYFyeSECIRDZlHJwZnH3tfe+qPL9z3reG+Z58CNNd9f+/y13OPffcoUNKVQApAPt5AP4dJGjd9T+QYjgLM7hiUfzzu8+KTZv/HL/5zRPxutNfprzQxDWzHAWwpwme+By+2/IAqSe1xQstxkKhEPfd/9u47fa7dHP5XTYJtuXa1SvjgQcfEKXmy1/8TPR0eTxq4tMYedJocg6Vv5+GryyHrxl5ibJKGpNzYuz65Mx8XH75dfGBD5wdC/p7Yt01N8Z9v35AaU2t1hbveudZ8Tcveb5UgNzZ4PWzUAva1h6okbsTWR8+H2tnQl/u9ncerkGRiSudiLtpvdy9WLjg39/X0EDf6UmdDnBhnDlmWfaeua7phbghrplOC2Vhk/BVFKr53+TBuV2Dk5h/j5/Hd+PDiaQB4S/72ndihoEOUYg1awfjnW99fTz0v1uj0jYff3X8WlFH8iTKzIIQ7JhoNA4cioosAfABVogqCXT4vcce2xQ33LBBCFmuiZLWHTG4ODY9+Yjwq0998rzo6eqQec+Fb0N/ZjVymCkhqqmNxU96ysJjpIfsrv6MkBErPPjw49FW6Yrjjz8yfnLnvXHLLaBULVFrr8Q73/bG+OsXnxBMBNOBorUkbRALlxvSvNHzMZfmQTCmRj+Hoh0WrJxq5GksEHPpWWPcFxaK59WluPAzH9Bw5PxFRKqCx5IjR7LOI1U8ExZ6J8ER/67xoU11VacfsO91O2emjKBMTMgc47s5GBSpucmXXHmTBxg2GnHssc+ONWtWaibCP7/7zT5YSWoPC8aDq1swUX0wzbIUktKzOaMGwKGRpH69Hk88sTmuumq99LWEtMksl2PlYH8s6m2NcqU9Xvbyl8vc85xiD6r+7HlJLD5Sh/ZzdlVsprHeZwAmuIYMgKh40ojPnH9xvOe974r9+/fFlVdc5c2ttcWZZ74uTjrppWJS8gdzz58sUGIeVkrjQMkSV4t/8t3zFC2ExbeZNy31O2BUfs/jeIgNStLLbETh0i+d1wAmhIEIdaSr3VrHWbCSsJybLXYf5vAZAwSFeWoo43xMT9G62BZtpAtQRPOMHtKooSFNaVbQkPpcr7r61pieqysXpSPulFeeGgt7W6Ov19oYfAZ5MvmsemPnLS9I4CBTmAKgjLGyqdR+M3l781N/josvvloLlAF9grMjlvfF2sGuWLhkWRx1zLGpUTu1qmjitYv+fJf8bMLORe1JbaeqIqnHiWJ6nnflAdMciief2ha1Sk+Mjw/F5z9/kcxytdYWZ5zxqjj9tJNFf82WgvdkkvaSJUv03Xr+BpPGcEOppygBKmTd6kxMbgGzrHJsGgcEmOPyX1IjuPhCFOTmdePUbVcuxdT0lFo4UXbjIQiQ1AgmUwVh2reD06yTnIrk+t+tqLrNij+kemkaboHvYzGA31iQT3/2yphJEzf57y/4y+PjNae+yN+RaK7Mqmvv7IoOdf2B+1YkvYB2IldVFodyJYOqEgmdlIf/9tRT2+KrX71GYpnCdyGYtbXFimX9ceTKnli5eo3+L4MFKNlNTdPF759VOsG/QWZLEom55dPIFT22ZplwgFgnlSgI6orFuPyya+PU014Tnz3/Av03eNinn/qKeN0Zr7EWFwFUElaxT6eEWJMlsb9HhMxUG/7dFbQ8Y8mFHd30dBhFrCikrsCCW1gKXzz/QzLL9huMDavo5sBkR/Hbzj0JRaZyGl/iyMw8JvnmFGXzd5hrlgb+EsOP9flsmMaFFgUXfur8K2Iaud96I1auWhnHH7M2XvLi45TL8jM8A9ZCUgAUtEuOQMXrFVQ6IT+oocDyxZ5BYEGVYuzcuSs+97krgiGWecPowlu2uC9OeO6KWLpsmcRHmd2jZjANIMbMH564hQBJ5imbVWi1ujmIb+IZG2RDnslRr1Ey/Px3bt4Y07P1+MlPfpIsWjle/rK/jre97cwotvo9OA7auLTZYohyaUg99Tm4uYo4aiqpaENTMJUyAzaVOEP7xHgbPYO5z4WvfP4jDaU1QnFKQkkoqzHRS3oUSZ+KDcrSsyTKUF/UvJSCCnGOEueWVIHPdGOSzRzRs0VAZ1SD/dwX18UErSlRiH86+92xuL81OttLIpVxKjGx5Lxq6m7j8JjPjPnVgqTFbE1AP+NWslwB3zd8aDg+89lLAi1L/DJ5rTZ3SV/87QuP0fTKvoEBpWaKUDWVy9MsiSsIpGTmEgPCEkw+YKqhAu8lYZU8clUSi0qQC7F1247Yu288Lr30Uh1wbu7fvPj58c5/fKtKc6r8JI0rgCEdklQRkzVIU8fNscpDJ3NRwyp8afxhsxzoqljOXmaicMVXPi4dKh4Kk4Z/9W21U9ZocfXPOnI0q9AviJkEKeLXOQhssG+xA56sNWX/WU3mzg1hnz7/yhif8dTLcz/60VgyUIxSSyGmZ2d0uPoWLFDNFoyWZ8L/aBpYkj5QHXaGIMcLRUWFQ8PB43uph55/wWUxpRl4vFtZm7t0cW+c8rK/VBMWsgNW4TEYwmJZSTUR0xKZnYzAfcHuJsQW5Ll9OfVyAcXrxQ0kkPvfh/8YV1x5pVwIEe6JJzw33vf+s5s9TWDoziiy9rMtmxl769YiAAAgAElEQVSYMIzd2c8ni76T/i7PtufvFVhWnBK6puvUT5t8xcWfaDQ1m0iIRfWkrdJ0SY9Ys4S8u9Dh3M66gUmO3YGFe1Q9X44/mORnNk7h/JVvIgJdr8f/+/evxJhkaatx7sc+Fov66zF2aEQRMA9Mr7BHx+SgIZ3mCLEf2AwgwGzGKYPhUwFhOO2ga5/57GUxMjbheTutJRVA6P059aQXqNQHFVX12/mkhJP0P9xVN2cWp0iCjhewMnlcTb4hmf2R6bHeABVkY9OmXfHlL18kwIG+4788/i/iQx96jw8An0Wem2YkONhMaquJdapjlEbeSXEoNaxlgdECtfZ02HMc5EawpOJ3+Vc+3uAH3F7JiJh2J84pFUpdI82e1rlZz//Jcgd0mOXc1g9qYjQbxC2m3IcP6ekDngTF8qH55Ke+EuPTpDjtce55H4uB3vmotvLzRsdo3VSvUNaqSowLNpXKCVPH5MPFUSrp1mkRod3A0hwbja9ccm3s2LVPmC3wIyALm/um1/2dwBh8Oe8iYlqLu/sNPXozC/h5xWM2d4IjU5NVdklKmdJomZxJqBbbUognn9wVV1xxhVJHRFD+4thj4rzz/sWxRKksbCHDjskuN62D9iTBouTtKiTI7QG3OkXzaFb7YT+Hg6+MDBa+dsknG8KErT+rBWBjah3tugl6NSoujF+bnpZEDoQwazxk9oNppCoU5IauUkn0zbk6oh0dMTY+IauAuaQQQSQ7OTWris4555wbyxYBt8FaKOgQVGASCsI0cMKLjU9MKHhSb4/gR9tkDY2se7ixfHFibV565bfjT1u3a4PYdN5n4YLueMdbXi1TTy0VtMv8dfqEAe0RyG7IghgBMvtK7kBiZYYpc1McdFyT7ljC1LQtHY1GPPrIlli/fn0cOHAwSuVCHHfss+Occz6oyWp5erZoOVLDoSrErEJH6+wJ79Vea4/hkWFZKxacw0jlCeAIHRO10yQmExbIsQ77NROFyy76RMNyfdYT5ISLPUBLBzcPotbERCxdulTVIk44p2RmZl6mDcFsmabUykGHnqimxaJKhZg+nhiGHxubzcjHzrsgJsanNVv9ox/5aCxfUo35xlyUEuDg0WUEcVYjb6YoSTtSXYVJKkHBXJpcPZfQNIKfb67fGI89sck3F/gRef4F3fGes1+vjc6N3hTuc7Gc71VLCykf35piEaFWSX2dzWdTsxg2SJZoOakYgM+da8zFk3/YGTfddHPs2LEjiq0NlUvPPedfzFcmfxf5kEFPcMYIXl15ymmVpmojuZBaR0VuYG/KdCWMezBUUttR0Jr0qHIWU/j6ZZ9WKgRFRtCVJnUoefUN0Ukg/3XjMTfJ7D8PW8x+QW0ZjUaMT0405W4lRFLEZKYx3o2GAA0i4X/71wtjZMLls5e+9CVx0stfENU2br4DOcBxeMOkShyUant7U5+Sg8rcXfylI3qLhanXVdpRxAzl+O737oyHfvuYbp6Vctqiv7czzv3I25vIDh2DROU51eCgEFRpYljJwtxN0yvV9CS9IMpvinGzFpbaUZK6bKMYjz+xJe677774zf3/rUj7yKPWxKc+9XFN8CKgyyU9tZYkjFhQabmkqhPxBH9wk2Qe5MOyTEWnUHTVcxCym8wUJUGPWLbrrvpcw3bfvlQ9BqkZS2kIeaqQEyfR83OU9KwWBxk7+2YWT62HqdSn/51aI1hwzDURnx6qWo3zPnZ+HBydFEdryZLF8dIXnxgnPu8YpQm69VOUGinFhWitznNJCTw1xGiRBUbYXH5Wf58avjq7uuOHd/4ifvHL+wV8cBg5ML09HfHes18nL2Q6aU0HoUNzAiiEU3EyqzLfXGezFs82rdRxBRSf3HjGQYZ1woFnHZ/asj1+9p//FYODg7Hhe7fpnVatWhH///xPqueIdQMPyGxGdhfLJhkJ6XM5Q2EdXMsGbm1TNgAC5fimoL9jH0zpTUKKKVcvfGvdhRpgwYv5yud2C4fj1EjVR5MMu6IxcM50mngpfEp3b7fMhKBHoLpWN5Kx2ZnZzw3mofiZCy74auzefyjaWsvx3OOeEyef8uroKE1EpcatsXAXQRNRudRcsS5TruNart6fpdIblJtJuvc8/4fn5TnvuudXcc+99zmnlPVpi96e9njXW08RWMPAqqlpUiCrzqFpqVSQyLpWU6TsAoXLb4pyBR7Yt4pOoxTJh0yXWe2Thbj7rl/Ek5v+EC984Qvjqm+s0+KvWb0yPvvZT0dXVy2GhoZlJa0DYkHUGTKAZA2zKAsXi98dGRluSihitbhg7AnW1paUy+bZ9jkYK3zj8s8oHBCzcWpSL81mOGiyVK3TIXJB8lxKbTAHHBkrQpyvR5t+D0wWbJnfM0WVG0fHHl+sYjwR38xsXPD5i2PX3gNRLpbjwx9+TzzxxJZYc8SiWL4M1RoHL/xhw/IGUzfeu3ev9DK0Cdinguur1pNwGqBaaKMev/zVA7Hxhz9TMxoBknhKlN7eepLSNHBzyGjcYKJ2qin0/XCbqrV2WSKbusOFAo8P9zu2VRFMcQHfPGRGyoCDRzz88GNRq1ViYMGC+MS/fVLPtfKIwfj8hedHS4u5UKp2qHPSsCLsC269eFIaalV38b5YDDQxGKTFH4AbAr/2WodQxNQn08xxcR0iSXz76i80aD/MugwEVjJzfDjguOiTnA7fZAMSqcFXzp++nE5JsJsNYEiQRcMMk3dmv0zUDcOScP7iS74R23fviUqpEv963nvjxhu/H2e99R+iF+hZs919w4m0eWHMKoeHE4xp6u52HxDfmRP47BtJibhRVIZu+/69RrpS/FCptsQ/ve1UFUrE7i8CX1abKY6EuyWQAk5r4W3VcBMaJX3LBNwjXpK/MwMMCKCOj87ENddeHeec8xGt5Xv++f26AIMrl8dFF34uGkHPj91W/oPF4T3tX3Mp0WAEkb7BIuSZrL1sEkESWKG4X2zVhmtuYhL1Ltx43UUNC3OWFF6Xy3SWm/nnzYIX7NZ/+kYBK3RalPsVdDoBIiQhkBRMKQ6MMaPA116mJpsLXobFuuTyazSsotZWiw+890xNF/uvBx6J5x1/bAwuxRWgc2grwiGhcsIt4tbyd0j7sLlYmIwaWU+CcWkuLz65aUt897afKl4gC2ABKrVivOONr9B7UkaEostIUh8SF0HIb6VYR8dg2gDWCHCEf8/mlFQpuxwzGouxdeuO+PEdd8Xb336Wepx41ne/933a3OVHLNPmgmJiFXL0mw+LmRgek6q20EpF5VLKqiY6uLmcPF8pExZklqknUJc8vkCHQa4ponDbTVcooKIMhR03V4gI0f4lvyA3iS/LQUvm1OKrOHFtWmTXI3Px2g/UKlYeXGRwWqZdYUavvubmeGLTluiqtMXHPnq2qCL33vvrWHX0cdFdbY3B5QsSvUX3XsGHTWBYOq8R2vDublTvOjVXl5vu0eahnHj79t1xy4afyUVIGbbYGl2dlXjzGS+JWhXFnPbo6EKEOssUulwpyX9Sm4KDOUGTIsfbcgF2OKBIWG9KUcbHZuPn//mLmKtPxRvf8IbUUdgS73//h3SgB48YjAsvPF9Wg5M/OQmpPYMQHr7lC9Ou95X0RJLzh+gAzSdnCCILJKYIBEe12Kg4Yw4b0XbhezdeJoKpBKoS1CdoTwCCo0bTXAx1wV/i31lA1xYdXM3MGZxYtmy5vlRISjrZjsI99NG12Hpc+82b4/E//Endbx8/9/2+gfWIy9etj1effFqsWb0wquXDCuYuS1ZjbGzEgwwFcszohCoaxxUkAp2Ck9nZ2L1nf9x4y13KYXl+yGadHW3x9rNOjo6aOwlJ1Ui3yMmbIqFi9JdkjXItOKdE3GzeTd+XgkP2GZbjw799NO6777/iXz78fgWBSsPrLfHBD3xYF2D54PL40kWfU/6uOYEauGUwiD9YD7+XN1nios/4O8CLbFXd7ul2HPnYeSpJCY7MYtobvvM1Fw7SjeNLpP2oWiKVHHOVMMVGP5gdO6taJhvFz7Ix/GyTHZF4vj4YIXpNxl5VdKjXY9vWrbFz1+7oW9AXq1etSrpLjWhpbYsvfXldnHba6XHM0YNRZZZ6fTZqKKWl5J2FBtJjE4FNSSF4BoIq/h1RL5750NBwXL/+R6L4SNuqWonuTohqr1eQpzE5CZhQLFExjUc+HCy3DMo2rk2kfUVwqhaR90LE2mnR+NhMPPro7+Pee++Oj3z0g3JVuVpWiNb4xMf/LQ4eGpJKzhe/xOY6bWlmESmdA2RRICTucpuyA8wzJp3Lpg1n5JuQQlJLeGtGEVXUIYNgzTMv+tb1lzdELEu3zISvurjJuYubB6VAQITJy2fmXyavZTOc8z/8APnZMwEAfoaH1dDf+Xps3/G0ivDINbAR9vdtMTS0Pzo6++Orl18fz3/+i+LEE46Ovt5296zOzcfY+IjMMM9AoLFr1y49LzeFP4JPJR/EcMS5uH79D2OCNElcq1J0dVbj7He+VpGpaLbPaNfALTE2tRnYlK1Kx3OJz5ZaJ22N2eCS+oX/56FH4v7774+PnPO+JJKW0sAW+m8744Mf+FAcOID240Bc9OULFRhlSyimadYdyaNuyD5IdVJ8kl3dFHOJ0ubx3NxAbrdz4xZRmIztG1coXL/uC43FixanvyBJt37gxOh4MzJD21fIVWpUyj+DKRMMl6JHdc9J3dQpk4YZzjvvhVVpAe45pTPZd6xYuSpBcczEm20qqs3XW+Ky//hW9PUviBe98MQ4es2SmJocVx5M8bqvv1+5ImU81E8zJJjn22rTWgpx2ZU3xvikc2Heo6NWjnf9w2tjYGBAZpDDkE0iroaasTUmXIwXBJjqymQPNGMbu8ViFOKnd98TW7c8Feec+6Go1gw28L4cZv4ft+nBB++PQ+DLldZ42d+dpMNoGo/RN2chs4JHczpJNI1lMBPD7gydL1nOJBHhHNzkOy5HTk1zbb3ww9uvkVk2m97SBsBvEEj4ZYIrC1dZOlesjIQGcdI1PLnOdBMYjjbdImwn9XFVh+iKB/RXw/G0UhlTbnoNKzKmrLtL0ThkbNU4pTdYjFtu/XHs2j0Sa5+1Ip573NpYQuNWgd4cZueYl8ULDg8NC3DRxJOWol6WA3Tpf9wk5TWX7ZDqa41/fMfpsWjhQhcUUrGAzxHe3Eb5sqbPW7DQ2sduxmqJuZiL+hyTtCO2bdsev/zlL2NgoD/OPOuNCTU6zD3m90QFKrXG44/+TjQluNUnPP9FTUvDuucoXRutbj74U6bLQDLMwJKxA/fdUmVTPJMuE01meUPlVmCkAgPf/O1LG8pbi8U09jONziYNSAiQgHFOLLhvKv+7aE7EN5UI0dMKdAjbJUAy74ZhiuGAC/v37dOpOzR0UH5xQB3mjVi5crXnrNcdWec0h8NGGsBz7dixO27b8DPJNKxZtTxecOJzYqCvxwBDoSGUxiqsJT8PEa0sSktcff2tsWv3QQV+/FxXT0e84y2nRnvNIuAq7Kfp1ZmI3tVpojqWplgmYkW6ELEXNDL2xYMP/k9s3fqnePc/vTOetXaNUi+R+Klli9xgwoIGXMxOxaY//EGb29PXJz3NCKNSGVkSMKHnSHL6Sf/ZXRu+eNILQY4idWlYEcB7wkXE/0J0MFkiZSwbbvm6UiE+XKdX7YQ8pDX5M6OC28xXGHpM83VSasAX5bxtfHRUEZ/Gqul0hczhof0H3Cg8NqLvGUBnWNCmF4XwP5vxjGKxcWywI/Ji3P/Ab+O3j2wSMrSgtytOesVLY3DZgNoz84wizNv+ffulicjNvOHmH8VTT/05oOEgwQBI85Y3nxJLlyz07CECFkXiHtki/i+pk7oIJ8EtY3y8Hps3Px2P/O6R2H9gf5xwwrFxyitfkVosnX6x6GDxuKrcH0VHYdTnYvOmTbF3755YuHhxLFm+QmVToNUsKvrMejgbbUaFZ0mII1ZG/WY8GokNSVsMuT8xjBLFhGRhxjO5T4HZxtvWNQjtnfySOJOv1mNijLxyRo6ZL+MmiPGnNANtf1daODHQPkZGhx1AJVOjIQtiNrh8dnD/AZnJp57apMIzs17FhNQsAKcCsC4PC1t6OHGOZvUs+Kl6Me6661fx8OO/14a1lVti1crBOPGvnhOLFvZZh3K+oQPWUirGLbfdG48+9oSCp7KgvEac/a43RXt7RagVNWYLiZiByEhyZtOODE/Erl0H4v4HH4rZRot0GU983nPilJNfHgWaxNNYWuehXjv5SwIhSSfBSKEYMxGHDhyQ9GJvf3+sfdaR0TewUNF+FRVb/qRYxkmLCW6sOYdeGYrIf1PNKpHgVakFUcHTUF/dbgY5qmEvz1P8zg2XNUgjFACk/1PxeCZFnNPTCjLc3m86aW7r5ws8MIl/msqaSe0ziSVP1If/kq+YnY3hkYPR19sb07Nz6rwnt8U/sHnIy7LP9smHU65MAlBRHpI6o8BLlXjs8afip/f+XLVllSaT9tWKFQtjxbLFcdTRR8U9//nreOSRJ6MVamylIhLgmW96paJmbixMkvGJ6RgaHonNm7fGrj3DcWh4REEKdexCzMfb33ZmrF69LOp0GQ4P+1A23JFIRQZlAJ6b2AHVO7olSf/w3+PjozGpQLIeB4eGtLldvX1O3yq1GBkelvqqAynPeRifcPus4omkLMQl0rAMNQiYs4YL0ESwkiFfsgPcJT8rct+PNlzb4Afk75LtF84854kY0l0SI9+nRYhKChRcS5yWL0PpJRf7lRql5qYJlNLA/xJTw81VrarScCrxTwQ/mBjXfdt0ewnCZFoCQjf004YgR1NZ3PRkxAzNw0I89vun4le/+u/Yd2BEFFVAdkjo0xPjMTKG+KYlhSptJXXnVdtr0dnemdyCx8qQP46PjcSRR66Mk0/+exX2uzraBdxk9XLl2ONjuvFoOrqFlJ5mw3/kwNKXFKhCkDop1/Loo4/G4LLl0d3fH30LFqZ2FNLK2ah1eraBGNIKqtyPxObxT6yBOh9Krt1ygQj+ZmYxyw3JTOkmJ91LiBbJLF/d4C8ymsQPE5TwwDnUzqF7ng59WIoezSaoLdZ9EvICZ0opkDm/+NIDB/ZrkdCiYHMo1hdLPoGUyCRmeWhIL5IrPlwFctHRkbGkUwFGPS3qjjr20sayoHwfgdzeffuUttDMzHy7rduejsd//6d47InNWij1KVGlqlkFtbenO444YkUsXbIoBlcsFSxIZqIyWuqwAOxQc7OYn4AJM+IJKwhN5dE6lSKCuiSDT01YtBgotsNDWhcmZvZ0dUWlo0NaGD3M3hOhviwLYL9tK0umoExl2sIzEi9VvEOQ5uY5U3Psqvh+4Fturoh8muEwx829RpubqxvGUQnL3VyEqfGwB7PrXSR2S7xqt3Nu4xhHuoAJI2XTS1XCam8P+nJlRqYt0FVt7zQlJ0JBAptp2g7tKM4x6SVS81MSW8m8Jvtg00fZ5MzG55Dz+2Ojo8pn1ZBcLEZ/f1/87vEn46bv3hlziWRQrZbj7We+KtprzL0jf/cgDMaxuckNpqKB+tzsRlDIjdHMwVZ6ZtubFbA8IZRnlLYI8QkxiJreXBvn8D700EP6zGfhcxcuVlGBdWJNxS3T95qg19vTE6Mjo+4lKhRiYmJMLitHyKwxPz8NAxVyRRInEx6RVNflyu/4/nUNpwKOGo0+ldy1njbSXXyT0dPd08RfiQp141tdUHAJqyDfZoTHCTobAIeI7eS/d3T1aFEz+Sxjq5l54EnWeeaBC88ug0GLLSlwy37fOR/QY00lMZ6J/wZahZlHh+L3m7fE+pt/LLVYNg02w1mvf4Wk7TmhC/oXHF605AoyzCi6j6QAXUGy66H86JSNnRH1SCPXSMtdjnMBvxAIkZC3c8sefewxHeRly5ZJ3ompJBnBM+m8LjEyPitPK+O9jdyl8XUMt8Q9JgQum+2WBP1ijnN2I+xiw/e+oVRI00USrswLQX/hJHqzHWwR4VmTsBQzk9PaaPfJWNBSjD5pJxrEyKeLi44oprvIXcpqpYEYYtgU/gXGR28a4lhOdBObIwSpYXosXz6oRdVph/SOH5diGtrP9veMcMkN1L7lEX/asj2uX79RM4ow3ZAR3vLGk2NBX48YFyBebJQygtRZyHPlQyuhaoECk1FG/IsbpizBtetM3eX9XTFi6IfrrUTuQ4eGYueu7fHnP29XoWLBgoFYtXqNY4pnjKXjM2dnD/O13PSGtZvVM7P2bDzfkzMSXtB5r9mZIlWkdhqdve/ftk7CntZhMlFMudN8XaaDG+HOOn8INwkTNDPll6t1dNi5z1helg57T/ParxuEBQCtgYCnh+toN54rcQ8qH5i8aeW9+Hoic/UJUbeEPdneEdMzs9HR1a3P4/+kFVWvx9Nbt8TY2JCenTRKQUnDaZCCOGSO9gzFlVffHLOzNDF7VuBb33RKLOjvNX010XEzJouLyf8701XQ3RodH9eBoPKFRSBG4FBhKgk42Qz+AE5QC2YtMJuYZ5rQsXwwOdF+ZFwbMw+wYrmbMo3A0lqoDZZDQnqW5i5kIiDfAaae1dolsq3h1VNRSoEUtCDVC26/9evKMuv01CheM43G8GGoXkoqMzo2lpqumU7t+XI2l3BsXaVg06xsSjdCi3wqEzj4IBUfCLCqbleZnHYw4LFtHneDNJE69hoOXGBacuMWLxvU3wkooAsAxZiWhroKDu3fqwX00IqCfBMBjUjlEVIE+NJXrxEWTPN1tb0Sr33138aigX7dnp7eHk+lfuZYmaQU0GzLSOU4aTPPQoofE3SKj7ceh0EgWCMc7NxkvnvPblmamZmpWLFiRezZsycmJ2di9Zq1SQW94pl8Wk8ICGNaK/hboHYcPFo7ucGkThwk1qVKayvPqG7DeTFVdVHSbCYCOG514bZbv96QfN9s6hBXl4s3iN3XeOxE2+BUOWWiAbgqVr8rGqbBajLX/NzhchxMRIECDtg0gCn5Z2biEBTB3ZIgSRUz5A52kQUUEbTE0mUrolRp1wnmsPB/u3Zuj+VLlsgXDQ8dFBmAiJ2WUz1zjheQMxwbjS999dqYmmJzbYZPf9XfSC5hydKlzc3NN8j8K+fkHEKicvGKxdk2diy9S23iaHM92FDPyE1+uqUltm3bpjhg6bIlsmQiRczXo1rriMVLl0isjc/hUnCgodlyqYhNSH/yHgguBOCgo099wh7Uwd6w2ehYyXzTAqpukZQK/egH32wQfCCK7ZGqrmwgFol/wCy7pAdpnYFKBvbVPplmACFVPzk+FiOjQ03mXSOxKTVZKyFgPCxiKSwewD/cXVIlTIq1lezbuX38gU2xd+++6O3tiwWMnSmVY3j4UGzbwqTK0ZRSGVVTdSXxnXNwtnfPHvGtL7rk6hiHAE9Nt1aON77276OnuyO6OruVbuUSYq6aiyguVgcVGNNo2VTAEw5Ppv6Qa2fSAK5LzeiFFo3AUycD0OPmzVLR8XxEZvC1Rzsupr09uvv6rZ8soVDrWWb1VQ4xt5obWyqmeYe0ZqaigQ5Z+Dl5X12e1PmAWebzCxtvv84q01RyZv2DmE9aDjlBubri9gfrL4HKZFmD7m6GPpVidHgoEOFUHqiHddqEjzKDz+aLNou+3r6YmDStU4A/PgNp+QRvZjl4V6sKMToyImxaJjCV3FRAb3MBPleVci2aaJzAj/RsenI6rrrmO7Fv35AWr9LeFm8+46RYONCr4I6xdsq71RJpRgPvw8GSqjryQSnPxP3kMNn1aW5Ym7oSxemer3t4dDjARBrxiSd+L74W74H1wMwuXrJMm00Kg3lljTHzWCDiDYInngn3oui/VtXPo1qQSREOpDz/QD1PHB5RjGDLWOWg8MMN1zcUfU4YhalWs2RBmyoZqndi32dmFDFax8H/vmrVKgU8nE7aQPgcbjc+m6ER/KxUv0utqojwOcNDI3rR7p4+HSL1xSaslAfUYsKISMLRmH5eBI6U6pjpZuOTKA6wocg9cMoB4zMZjxvFIlGd+vo1t8SePQeitchhKGlzV69y9K2UqbNLv0daBJpEn5SxXbMLCfI0GmZuTsEj0SrP5XabOflVnotJ1QSMOYXk5hLpT0+66lVsrWgTOey8oyR4+bxWV+TIubmPE6Muieb8Hzkl5dCoywKIpqZ3flc/l0qcUhdIbZxSI/jB7deqnlsm9ZGMgXtmM5WVxbfAiTk+ueyX/S0zB4hgDx7YZ1M6Pmo6ykzq8puDZmo/ygJpUAPiWZ1dghA56USlvAiHiWcxO8EFB4PklN8mhNbolvFMw8CMlngQAb7FVBM+mxuH/1WHw/xcXPftDfHHP26NEptbK8dpp/x1HHXkGuXHGfAXozM1YTGjQFzkxPTndmINmmPNyQogzjNJLJlVzDC/Q8CIqYdnjGAKPT0QCowh9zsmAI/u7oqWNHiaFhxuGpNVsAZkEE2cnxEFne2yXnxOphflg6XZSiVrhRAfGAwyXaiwccN12lxJ/qlTLaltq1hBEAS1dNbtkZySFNXx5STkTz/9tDZFJbaEpQouSz021n+wbgU0HfplFfEy/Cj142Rcm81Ca1L549ys/HGOkPlsQ42AJSbzyYwnoJxIM6dAdM0bGTKRbf3NG+JhigfFclSq5Xjtq18aRwwuEzKE1jO3hk46VWRa0GlEms+SBTyT2jWS7D23hXnCfC8MSt4d8y6LhRJrqbXZ6QiyhDmVel6K/hcvXtQkm9N6yrvO5hl+KdceOnioqSzn3Ns3u1atyAV4GLS7JKgDtNfod3LQyppyqNRk9pM71jcUrRHJcaWhTKcubhZT8gFq+rKqKTgmL030dwA/WCzGEqY+J1CCk4p5pGSofLlhMRUWmsUktREjY8awX4tm1jsyNDF7UkEb0KF8qDr4qBSNNs2w5XksmUuuqQJ1KnNxczCTkN1UpZqdjTvv+mXc95vfaXOrtVK86XWY5RVC1fge4gFcjiotGlPuIIqCNdEAABbUSURBVM0d/XMqBJgu6qpLHqRM8zQ3QoFouU0XoMlWEYlvWN/BbWMtmUec6+ZYLAAgLgUVslxb5u9HhoYT1OspYNSgcVnkvUpBk04W1tCYdsiicYDYD/oAhCXc/eObGrzU6LCHBhoZsY6gJ1TNyexyQlVISOE4IAaBAD2uPLx+D5nAJH7d2e7wHCK1JmOmP5xSBQsT0wqGqM7wObkowWcoqFFXG3kzAV4aClzA7E/osPC9RoscjMkfJq0qvlcaWbiHej3u/tmv475f/4/MIHpQZ7zmFfGcY9Y2p2qZAGhMnRui9IIuhMQ8aZK/a4yaNWsCF6PJhPjl1E1KCsaaZXUAigbktlwOglssEfEKzwqYQa8xmzwxnuhJUqdpUf3Wz+/OyvaOmkCLiXFST6dDKpF2dSZKUx7HagAqm+zCxtuubUA4U7de6tHh4ZnHQ95FyS+T0XUTE+Md08HJJj3JPCDBkcm0gH+yaQQVbCY1W8kalK05wbRN/DZtKJhgsFaERa2A5pOMP5X+MSa6ah8q1Ep9QiZx87N8ftauIhd3Yds5M+yEBx56PH76018gO9Pc3GOOWp1Y/Zbpl3/WVBWoqhDc2bSGvleWgRw+NaILMxet1oeLw8cV5pYqF9btL8a+fXuULWAJMJOlkgMp+fO2imgxzG7AikkFr4T2FNWgGUOzsxYUHVi4wC0kRRrCRoReYeGUz0qm2IcOK5lr7QKSNt56tW6uiGxSUTMfGefND2RtX+G/XV3yHxq/MkfbBovvcZ/UGNlMugX5ff5uYGCBAAX+XYhUyco05JWYOvxk9re8LFSUFYMrtIh5Srb8fr0uU8vva4FTAJb6SIzyKOK0xZEphTzfUlCUvWnztth4x8+lD9VeadNQ5qOPWq2CvFV5qFsTmDlfHJ+wcCdrIhQOfa4K5UKvj2IF/pnYG1kpVlyq5hQ113Kh3sICEZUmjRbg+VkD3p1Dif6Vs4SK1g31G/5J9N2/oF/rKsL93IwqZgBIqhCJmOjxsLlIo9IfI+5gtdx+01UNHlTkciY9T0/pJbDbqtWmEWpgppg9FlSsANUqh5tsR5JmTAk1RuWAMDiqvqXudXXfqfKzlpYYn+JWm31AwJXNK88gwRJySD2HUSFH0yjR1eSP8tjyzH1y7Rn9qnKMUWZUW6VZmVu27IzbN94T86inVtri9a89OZ619ggtlH/f00AUcbZZsIzZgZDb+cNz4wYyW5H3E9I2Q/VrXhi8GSl2I+aKjem9+MyhgwfVuEYBQuVVMGg40ryLND1oban4QAtGNCsTd8MB4zPU1oK+c4Ztk1gJzwKnnN/jebAMGV0rrL/2yw0+iEWkIA2tkxPVWkpkscRJxs6rFRNtjNmZGD401AzXVbgumB5jnUTnhKQZqN8o0k0142oHSqdm9GFynQeXxUUmGdcMPoh5pFJQTsbHUzqUhFY4IMlcsoh8hgQ+U18u/TR077tWjFzgXBw4OBzXfnuDikgd7eU447ST49nPXit/B0GPeoNIgYnwRz6NOTZfuNGk4rKAgBM8n/JgSGozM7Fk8RIDPLPwoNu0KQaAxnQBvPmHg1MVMcDVISdAjk8HyikodCbq5+afsZZYpOXLlse+/XtS/m+oFcwf64T1JLjt6DRu76rcPI1g/0Hhvgkb4gsFBMhdGfznl0FLqEcafpyWWVY+q2L+XFTKsAQndBswE1gC2i37ehfIR+D7+G+M9cb/8gCcXDZH5lyi2I6cMW/4YPwr/zt3OWS+s9CX3EY56yhcwpzcQPlwgIVRFdXZiLHxqbj8qvUq2NMr9PrXvDKOPmpVdPd06X2klI7iqTBZuycOCH6QzccE8uw69OrxBX3iUIIBgCpVNC0UdQJVo5JkPf2+BKLqK0r4vNM8V+DUFZCmfmEZ8b1sFg1imbGCe+Fmbt22NU488a8UtFIlE3Eu1ZG5CHwPe+ZuzSn3Kt1zx/oG+DHSckqAK20xMjwi+NHS7y7z8YCSYAfoSMEKD5CpHtBy2KQsX8CB4cTNAFQgTZAFzMpuFcUnyMwrN0Zr0gVvzNMzhUSVYoB1p3GmPKPUbkQgBwefE5abu+V4lwxDZiYH7aSXXvnNmJ6bjc5ae5xx+knxvOOPU8O4ABONN6cwgFAZ07B9gNlYECV+4CAdAxqPaiDH0bnLk6RR5MaZP01hgQNDmZPn5fMsvOYblf0jvw+9lwMBA0VdA+pbsViYg0RPK+OS8d2rV69OAZjnPYkRmuYT8jOskyJ+JBju/P51DW5I9n9snnxtmHknjk4i95ASiNVHYFOva9P27mNqdD21QtjJW2mchUAjAxHrsqBDLEAWDRPLYJxJHER+0y5u1+uxeMlid8qT+6b5s7ycYUVShDEjQbWanoU80XRc01lIP+Qni8Wm3j/v9rWrb47JqWnpVrC5xx93bKDtyCIqqHNLnosPIEoj8KvT32emBV38siZT2mBMtEw5Mx4w11Kha6gSZilDSxCRcbiH2CCDLo2kkWgrdeVJNeS5ui6XJSwazfIl78UBIPImQqbFhmc21behAoy6FFtahD+INz03G4Uffm+dfC46URrP1ki+B+SjvV2LTGChoKK/P9UnZ2JkaCh1B3DLKwyttp2XfD6pTJKfr1QVGWaVG5iMripZ2oAHwrSxsZlhn6G3zM/NVBteIOeY7p4vKlDh0FjiwBpWmGS3WlhGmFru+ps3xghuo1qNN5zxyjju2GN0sKwtlaT1lZPjsxz0cIk46Ji9PAk0u6E8UlWBI4AEc4HSbSaqJd7QCDlx0uichPNl2hAN7XljMiHfgaoRNeW+E+M68ELZ4I436jE2OiGXNrh8UGvIcxM8Ug/gsKnNBzHwVPcu3HLDZWonQfZGYAIYbSKa5xPKqZHmRAsC2hNaSGij/L3lFoxsGQCZkpnCd7Povf2kQ7Ni+OE/ANaJeuH+Sje4jlYzaqvm3nJjMCksZmZdugJigS9utZuezMbnc/B5SpWkB+W0hufIbMThkdH43oa7Yv/BYZnlU1/1sjjxhOONmlVraeiFJQFznu0AyFG7UsM0KMIYsNs+RGhAOYD1aLOJZvNMKSrHnr27UzCYx7p6jSgQqBU0FUw0H1gTOU1Sz9RWK+HaYnGTWFOlZ4k/LnKEqnh+dtZB+5GKL4XvfutSlfx6uo34QJPhxGjiJGYoKZtjfkTZbHNHGUOK+KNgi2qRBld4Fp279ayhAcWUm2tmR0OCIiwCP8dpzhsDZJk/S+aHCJqaJuYt63AQjKQWFx84sz8w5Rw6PTe3BTgvCW3y8nv27Iuf3P3z2Pyn7dHZUY03v+E1seqI5amTD0Idcw7Ugq7/lqsx1qZyWsc7a7BxCub4b1g2UYjwwzRsl+wneU8NPw5G0+2N/t4el/hS7xWtNkazKNehAH9Yqt/iMEkLDJl8kdBbXK2qeo4SB1mjC2ZmdZMXLRxQCpvLsuIyo43xg+9+vQGg0NOdwPZZ837yxAwiXYMNANit3HkHN5H4wm0VN1fPz6ZNc88RD8Qpw+fiF7mNKjSXHXFyWDT3jnHj1HyroDcAItZZ3rVjh0VIkuRu3mTGsuB3iU5lIUqtSnl88tv0ghxCPpfDIS3L+fnYtu1p8ZgXL1oofefc/JYBBU0laQDeVNxUJZSL6k89Ors6zawMSzaIvEBUm/5bE1qdI0+uqILDc7MBkA0g1hnSteAm5D5pVs8mi0BTeHd3KuclPWWBIfQbt6lLEUvAuglyhaCYNKtEL4Luy7MDgkyaxcEeFb7/3asaon5UqjE/NxUVwPxyOfbuO6QPypxad5Mb8VEHndKO2ea0TPpbRCgTKX1GmC43KwuFEpxoUYqMPnPNkwdEUR1zKr4Vc4d0q6Fvply3XI6hYSZvesw69FodPjjEcLGUKszJ9zoNAwI06x9zevAAAUZLTI5NxM6dO6X1dOxfPNdiJ4q288icLG1rPUtKb6brWthbqujphvFeWAm7AmtTShoiTc4k0maRuU1KoQpFkxHqNLzVmmAJUGxmjuaCgipqUiJ07EIAxedzwZQDZ8pwCYnAMSNaaSpLHqhBYCcU75Zv2+eS4bfXLJgxJFJXIqmJWF0Q/0hOPA1B5AZqISUmYmFP/i4XINh8zFiudsAOkLYVJK+k72RTDCV2SkEQn0caBltBvUqMFoeNkIY8kI4YurTgtiNt6zYtXrxYFoPF5r/pnRqFGB4ZijHoP2ma9MT0dAwsXCQZImBLNhHTyB8fNkfuagNNcKclAX0480Jy0zgYmr1XYrxOh96BzVLcAGk8FVKgDfP7bK6bzlHRo5zoxm/HG20284yAt+6g05rpKanQcalECKCtVKPRoSGNmZHK/GKUBZLwJ9i0yrN3brimMa9RMo5iJ6cJu8ll7azpz2ER1bmuxBnkaqYJcuexLWMjI0ru4VHl0S1EfYw9E7pFGkRFgw7C5Bf5XMavHjx00KnNMOYdApmjz9z1l2UQ+H4WgBsIMsTPCQgoGKXJz5kpOyr7UcCQSAo6kvUolisxOLjCOtFJ/d2AhNs58iHFxzZH0rQU3cVPDt7uMiDP6/TH7smYMwMT6XsyqyXTktRDRGNb0p7KBwXGh7Fot14KXZqjsdwHmtZNU409CQaky9zlqqwZeySCfxqKicVwwAeXqxCFO25b16BLDJCbkzIpkjhTpkxh1SiXlLIIwEg6g6UKi0pjkiFAZHXwnUBnfKH6SVMEmIvoMtuopSWZPQ6Dos5UhKeFgiNJ4AC0xkLysnTOESRJKzHL86DRmCJsPgPzxz+59SJwM90D38lgyL27VROFHssc344OqkgGMHI5jigZ02cEyVIPCnpEyE8Dq8TOcETMd+WhURnUIH3Jne98BrFBDvTkPykgaJiFh1th3eSqhCdYicYWxN0eo2OkmW2aPsIBt+BbMbq6O2Xt4K+5R9cDvjj0lntwHl244/Z16hVCdAlucmb3WafRRWvMDLVD54zWF8wFAV4GIhrmkmBkZNgMSJfeppu4qkB3JIY6McNWUc8+UwyNEYP0+CeCq/zv/u4uRYbcSMF/mC9Mb5rbx4HA/+n2JhNJ7kxn4PDQUOzatSO6Ozv0e/CW+gcWGu9OnRGK8DVvwYx9ntOS9qb5AkMS2WJxGP+eSQDZTCu9STPtM5KWJZ24YULoMPVJYDyPhqFUJxeSmsZUoUqBFs9n9UM2q9B8P9aWvcB8c+j1LETXgpDdiUk+zX8r3LXxOnUcAD8SfeamKkwri2EqhyeRYMZ4Qb5AdNVUuG/qMqmDwDVFtXaWXd5zv4uDELVTarYdBG6CAksBI1oiykuCOMXWmPP0Tke81q/ys1js2lHhdPI7DvA0L1Cy/M75YPtPjNGKgV8rxcCiJdHd25fGh5uaYjw24dg0UqcAL7NDOPtiZUitzQ1kigcm7dsx62w6SjtKU6q12LV7t/NsjYvjorRoNCy/i5Xke8GS5VqymoEOHBG7LR/mV5vFDIZED86bbvlhsy05ZMIESgzlcoApHZONt35DHCqxIzBtdWCxolCObKJkpkS9sciYyGeahuk5PMKfk1wdneT2Xz753Ip8M0lZMHM8uEd7GxtmA+jqM2mbQcUz2rgsLsrpxiRBdQHpUvlRwzNGtTj8nbrTCwUR0WBG0p/Li06Mj8WhoUNacFRaeQaKF5L3SXxk470ukuQcHJNOJI7LOFxzdu9wVkf34EZbMQ4l5lmWrdASO3ftal4GlTWZ51f1QCzgRQETDbdioqpn1XnHDiBYxu9dm6aq4UNIL/N4dLTXRHQwv6oUa1avUVO41NOTGn29MePNlTmE01tpi0MHhy2igYNPPoAH5uEpJpgh6ZIYZpLNEPUFdGl4RGUn56QGyHHyHBznaEzT3qfbTKSMj+OU6vDMuWtcdNqKzXKT6ZEEScxlcnpln2agXBpUiZBNtC5+Un1em4pwda4mgQANDCwKRsRiBbKgadMMY6068O+Q8s0CzRYqayCb0+TAB542lo3bSfmRxVfBZHLK6VuS/ssDpsrFkpC3fAFoDQWpysBOzoPhWlGoBxThgkh/szktzP27fKYCyFTrzmgeMYFr3fNR+OY3vtCgDYKolgdn95XfdnQ2WwxZyBnEP5SSWEzSnF4n3AQO8H4oKM/XvQGc8BxI6XRmFXFLs4iZYdNpk2UFUg+cYvNFwk5oDw9LZKiBFlm1NHG9+B0FYmoGo4vfpHIRBqbcp7Rz924dLDoF1anfXhNoIHM2N6+N4Rk7EzmdjVUaRzXo4CH5W8kEthJo2mpJTiiRElTbncPiOLfGenCYPSDa0CHrQYEAK0bUrJJnB5TVUYEkOd3LLJNML2Z9BHwkcXK+k0BUUDGYBDLEDOVKBRBLSxgdLGy4+WsNMec0fwdFVeeXLZiG1FKhwGfCqBBjx9lcggwWxCquaC5ZvrelleZjK3xnOogWYQLNSPsu/vDinLyJcZt7KJsEb4YaaRAz1QCTRhGfQY8EbmhLqqyXGr/4PE454AkFDtRyNAMQHHxsLDrp6B8dFXHb/F7Pn+WQLBoY0K1mQ1gkNj1rPdpfqpimm2PL4IXjv3taiEuiedo068ZaQB7UjSvZWqkIgPYkHY6ow6kC1lAJMqvycRg4lCrCFFv1rlhTrCaWyMwON4nzjBqCOQWfzFL4agTAwgrUqMbBgweicPePbmhgVpjVqmoI0kFJXIwFwAdgkgmm3AnuF84Do/wAU2kaJ7TLaZPKmJCZ5guRoI+NDqssiLimyndpOAPxqPpl1Id7QOaSPHRYNWZHilIjTdLEmDJTbxzwcbuBFyGBa3R6S4u67+jrwb3gv4kRPNXE42UkCNKaBjbR2Y60ktI2k7o5hXyulGmSzgS8Zg4pG2BV9JaAg0wzmJqnobKOuK+KYrveKSmYYwXgUmXdK9bBJUwiXEJi0rRMj/EUFck/iRljsRlubhYQB3dXNiNgadqST2hRSfGH7sY0nu+ujd9q8ItZgr1WgaNUUBWHm8uDiTucVOMI43MuxemUlpIK3WmI47zTFZlthVvAjCTX7taHa6XitArkMyKpQ/NEPk+mCnAcjFhyhPivGUn50R/rG02JkGDCB0/MC/F+DRtSz4Xch0kmAlapDYgQacCOTp14IE82OLNJNCkk5Z/qOpDuogNCddTjqnAtSUmARjUzMyk1eo127NgerB23lGY1PRtq6m2VWLCgPzb/cbNlkWh2SywSUhbnu1YI4v8jaOQ9lZ5ChxVo4oBPaBaVokSSZzyPhdFyPp6HOnrIRuGeH92gwgEFYTdrWaJgaoq5NvCmKgq5McFWaHVFBxO7bx8N1q5q0N7R3U3x2qWwnOBv37lbYHtfT5cgNLhD6iJAnHtyIsZI/KMQHTUDFckli5bD7cC3YN5dv2yRSKc62ATbeYgG1oQ2lozw8PL4MlReVZ5MPKtc1Oef8Ke5TZx0eoRwK7kBDTegHJcJpJWKGSipiK9iSB79ngVLILSrIR1kqaFigdpUwu0veo8US2Ca0eRyyykxB7RWi5Ga392QTyUv5tmZOk7vkGYORZaFSi03PJ82mBiDuMXFmQyKKFpW8JPSm1yaYnMV0GhwYVUQoZulLf6ZKaT4NiJg2JBEd/wT3yzuVa0qnrLIckWzENRjQ4UEuSIA+rlZLcDUuBEmtWOSLqWmM35HeCr4aVeXhDU1NFFj3TxnlvRq755dnk1QqcShgwdlbVQZQd62Qk5MxwAqNHy+5/JZbaemETfc6FwnFXcqcZ4wwbikLGBqQoMPO89gfShbIUiC/EG4VNapUDThoVySqt2ixYvdqK54hsoTjXVzUg0Q3AiWLeTLBIcs3j3RBGhMoNNUtukpN6ylgIv9A2Qy6maK7v8BHX1Jnb0Jj5QAAAAASUVORK5CYII=">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -536,7 +551,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1038" name="AutoShape 14" descr="data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAHsAAACkCAYAAAC3r1GFAAAgAElEQVR4Xmy9B5Sl2VUe+t0c6t7KVZ3TdPfM9ISePIqDRhqhZAn8DMu8hXnPmGXAawHCZDDmwUMYk0GABcY2wQSBSBaSQBKDNJpRGk3OQTOdu7q6ctXN8X/r+/bet+7o+fbqVene/z//Ofvs8O1v75P6ylfuTwaDATKZHDKZDIbDIdLpNHK5HJIkQSqVQqFQ0Fe++Du+n7/j116vh1KppM91u11kUmn0ul1ks1lUqlV0Ox19bjAcYjgcAAkwTPi9XYfXKxaLun7cm+/n/XuDvq7fbbfR6/X1Pl4jneZYEiCd1ec5Xv7ni9eIMfIavC7vw1fcg99zrNlMBvVaDYP+ABOVCjqdDiYnJ7G+vo7+cICpqSmUy2Vdj/95bSRpNJoN/Y3XHQx6+prLZFGv11CpVHQvpNN6P+eB9+X99Cz+lXPG8fErr93v9/X+mAP+rt1u6/7xe36en4n38JHHfx4MbL1qtZq+JgO7ZjabQbFYQurRRz+TJACyvtgcDC/A/5zAmKj4ykXW4g046fZ3CklMLNcAyVDvyWSymkDekO/JZCgIPc46uFx68H6fP6JSqaLZbCCTztjkcuFgg09RQAYDDJNE10mlbHIyubx+jjHwPrwff8eJiYnm2PL5/GjSY3K5yFxwjovCx89SkPj+drercU9MTIwm2+YgrbEUikXdo9Np6bq9Dt8/0PizuSz6w+FIiDlPMU6TBKDVauna/Bs/z+cZF8zYWHr+VErvp4A1Gg1sbW3pd5VK2TadhDBBqWRj5TU5tkzKNif/a30eeeSzCW9EqaBUhzRmMiaNsWt5gZAwDoSf4QXGX3wgTjDfpwE2GppkLn08kIQ+AbLSHKYN4sFarbYmm/fkq8MBZzJoN1vo8/tsVg+RzmYwMzOja8YYOAl8qPHdHRPJa8Ru5vslKJkMEkp9xrQDBW44sPFo0pEaCXOz0USn28G+ffuktXRPLnCvp89QSMoTpp14T16f8xC7lb/jz3x/aAj+HEKgsQ+GWshWp439+/ePtGyMnfcZ9Hsab284sE3A3ZskyOZMI+dzuxsxFlnP0uuaUHGxbQdkkMvGg6eQplhwx2ezI9XDwYeKp3qhpPPv8Qq1rxtQLfUHSHH3+04P6YWEwXYIP8Ndwr/x//b2ttTOxEQF2byZEk5Es9mUFOt+aVPNMRG8X71eH/0cE8txUfXHK8yGFjpJkKdK5GK128hkM0hzTLwfhaBQ1L34GalvQIuhuTIjos/SJHXaHZTKBY2fgspdSIEYN4tUrRT8MIn8Wwidmb8U2u0OUukU8oXCyByFidI4+n3kc3kMYLs1TClNCe/ZbpugmrkbjjZNMZ8zIX7mmYcT7hqqU74K+bzZwIxJTbw4UP6ev6OEUgVJsoecexOOUCGyYbk8qKz5no3NdQ2CExFmQjug29X1ymWqnwES3xm0vnpwV/cxCqp1jqPX7vBxkc3nJQSctGq1OhrruI2L3c3J54Rwgig81CBSdy5wOZoPJBgkplI5YVxYCdtwiKYvYJg3PsfOzo7uqUV0/6DdbWsecrmChIjCzvmlLdd8pmyhzBylpJK5cfjM3ADtTlv+QzzDxsbGSHiq5Qn9jf7EuGngfIdW4XxwLkJ1x9+kbb/ylQeSMp0E38X8pe1YU9vhjPHBeSHZJ19sk54JORJUg8WiSbfZNu6+oSai26V6tuuFitNuGZrTw50sByudNtua0KY1sb21je2dHZSKRRw6dAirG+taBNpH2ihKeKjDuG44llxYTmjsjBi33i/NQ7tb0PWnJie1O+kzFMsVrK+tI1/IY35+fuRvxFyMa69mo4Ecn6/T0Rj17IlNfKfTs53X72sjcY6pwQqFnNQ+BWVlZUXjp/ks5vJaAy4kf8c55e/54nzKbGbMNNCMhXaKv8VGDBPKcfLznA9qPdnsxx57KOGH292+VEkpbxKdSnEf8UY2aDpwox3mNjkmOLzyojsLcsiovodDPSQH1u31sLW5qZv2B2aLudgUECrJGKQW39XpoD+UWjOv1zx/Si2FiLuF+jSdzqDb77k3PpQnigGwuGcR9Tq95kk5W/Ja+wOZjjTv7d5uJksHic5kHu1WC8ikJQx93y0lqdTE7pGixkvrs7LJYcYonM0mVldXUCwUtfuSlO14037uZfNGqZTsLn0AzpG0B4Bex7QOhY8CxMXms/Kz1CKT1arMDl+r6+t6Xr4nbDMFM3yEiFBC8MOZTj355BcTqhpkslJFGdDB4ETa0vZ6HQ2aaom2iu/lhHJgfJBQY1IX3M30SD2Ei5Aq7DE93xAgqTEP7ai+5Xi5d08JplXs9xP5EXxY7cApk9R+zx2gQR/JMNEC8R5JYiGWpCexHVEsFTHw8IxmI5fNabHtfnwiap8ChoNEO3B9Y10LMj83p5+7rbZMVofOkdtwOUU+rjATw56ZQfkrFNi8LUy300V/0Nd9ad/Hwz9+Nmx4q1GX2s8Vzcni83CMVPGcf96v1WhKC4bDG+8L7ztsdcyjaVWLKjS2Z198IqFNkgT1uihkcpK8YWKhQKgLTjofIn7mLih76KAwhwvsNl5T6HFpSLWkjB6jS608U9nOtNSSpLvXe02IRBulsML/ZuaFXrTZPE6IHoKeJr33rsX0nFhei3aWO4LPxWeKUIy7k2q81W5pJ4a3TO3DBdGOTZuqDDVqiwp0JVR2fwvV0nouhYa01VzU4RCFcmm0q/nMNCvhryhUpUD7HAlTGPakbrm4IQAjjZBOj6KWcDLNL8iNsIoILWOueL/Qlvydnv2p5x4RqFIulc1uwzzbcqkgCTdny8IVOSeuiqhCQqJ4oXBcQm3JexwMMOngQ3jo3FUCWuiM0V9JpxRiUUVxYSOc4PWnJyfNi4Q5TXpQJCjkC/LaeX8+JD1pxrdcKKp4TmIsFEO8drulxZVJoK2mk0YB6nYNtODOd+eQO1iefio9MkXUAAp5ej20uh19nhM5HkoVsjkJlRwlmqGUCW84TvGZiGBoMrtde26Fn7Is5vxyTOHAUaD47KGyuXBzc3OvCWUjnAuVH+qb742/6XpPP/eogkw5LcMBCrk8mrU6si6hqbQF5IWCxb5STZykUsnCKk4Mna9koAGN7ARBAvfeIzzjoLk4dPT4PqpIDmK7XhvFvfzM7MwMWu32KKzLc6L7nDhDybiLqRppTkpFQ6K0A4e07ebwaVe4g8j7Npst/Z0mioJRqVb0lYLNC3KHc2KlGt1eT9BLdmSO9+ecMIwUltDrax6klRJaDQN6KMC8Hk0HJYoCxleYNOogaaFOR5+nNy6zZ2/D/PzsSKOG4JvDa6/xWJ6fD78gMA5uAqGh6YzubethplWLzZ2hsCABOq02qpWKSSehR/q83ClpAwG4GNyx3DGx66QmcqZqAjyhMNTq9dd486PY1uFBugU0B4VSUXZ0HC0at4+h8kIoQ7VucXfT4XEAQ0JZNGiXoZs8dtdMXCyzm4kBNPTUM1TBpgWIehEmrUwY3KmFpOYo5PUzr5dn3I+UaRIHXei48aXQldfu9qShKFjTMzOjiGZkN31M1BS8PwEbLUqhgEa9gYmKhad8hWoObcnn5FgVkfR6Ei5uHL4/5t6wCEMWBU7Rdxmak5h66tnHkoBAOVmUODpOmXQKDC3MVqX1gFT18pZztDe2k/h3gg0UgMCF+X6qND68QhXChfLOzRSYM2UOoL6nL0CwJLHYnrY2Yn/6CozZOdGESTWRdK40Jj68LZjtPBfIlMW2HCvtOHetoNax8E82t0sVaVJvCF0GRPEYslBI+FwMnbhr+ZwUBMW57plzgTkHfF5BpA558rliXqYqVY2NWobCymcNDcdn1Wd890tTMqZniOvQzfT0tASJG5DzEoJuzrAJGsdvttxQtRBwrolpV4tkUi+8/IwjaLsgCgdEEF0OBBfL1Qe9VvNg9QtHwMzrJfTJRaEKlQfoi0nEZ2NzwxElG8y41MbgLTGRlwoM3Jzf2QLaAyREy2lfAallhm2cVH7WJm4gf0A+RD6vhSKerJ3q3jd3KLUBF1DXSlnSRzsjbQ6p7bAKehJYe1ZeK9RqxNpyHtMGJnEX8sXvhTJms2hw0YQZ0GegYAwVj4dQclEnpyYtOeTTyvFwiiLMpRAqWnL7G5uEfku9sTNyOu3vKdn78MCZhyBIQ8xEavyZF59OtIiZFPIZokwNvbndaqBcKGEw6KPoWLW8c0mK2Sg+kOBFd3CUpZmYGDkFFBpqCmZcwqYp5u6YrZH5cODGMjp5CY2841xOmoVj4TWofQK14wSGdqA24WfDWYoIIkIcU30ptDud0b1kagbEx7N6BoEghCzTad2Ln+H9+BniCwZYDLBTq7lQM2IxRDGik1TWsk0Ubl6bfoZ2snvcMZ4AP8zh7KM6NWXJIvoXBT4/zUxfmkJ+1MCwBjqTvP7U9PTImTREzoQtwmD+bmS6uhQUcxilgV4++5KEiCBARmrUEBxmcxT0p2jPbUcRXOC2swU39IuCwt9x0gjtlcplhWHh2PDGdQL8zaYGPlGZ0OcD2aIzxJ/lpPCaA3P0qpOTI7+B15eEc9CDvsKi8GojpjR1Y1omJpYIFe0bNUCn05ZfEF5xqG6ZBU9cUBtQi0i1e+aI9k8qME3YNJGGKJWKSIa2kLy/wKVCVosRjlK/w4wefYMsCDYF3Mz3M2oggra1tY2Oe/Czs7MygxGXB6bPZxF27iqeP0sQ220JFneurunp1LDdYSIVy1PLyWY//1TCC+RyWYM23bGhyrTQimogh/Qw0c7iwwp6c4mykMrsnh6eNtRVeG1nR6B+2DA+CCVND5LQqelJYmWvlRk1eJYf53hGgMWQKnoXiTJNZHlzLmAAGgrhaNv1ecPCeT8JL737HLFuy3QxxuZX/p2LaGAPowWOlwtroVOnZ37G0L3xiCzCpvO5OW+0n51O10wLkbY0Q7WugKq+A1S6n4dk/IZhF6OOgKQjvOQut8RMSiqcY+dzxqbgnEYoK83nDhqvR/vOr1wzCgId5Ugppx596pEk0Cthub2+FpXOkGDPrCUMUkyMM1HiMabCINlXUyN0lCSBvnDcoRQMOkemWgwjpvetzJDwdMavGUkdFzqIArHLLRwkNErEzAAOLgr/zpBJpoC73L3rVqcjIeHc8p7joQntI69BoRHSlBhAxPHH/ahOI1mTTpl2IronGzow7TaO7UcsbOrUEibUVFqklAMy/S7o4kWem8/ATcB5irCJX/lZjpfzwu8j8rFM3FDzzh0aYaG0WJ+hZl/+CZ+DIhs+Q2g5aVHOMX2OrzzxsBabEs3kAzOblvUpyIYw7JG7z90c6kJwqKl0hWeesjTPkHivQYMCMnyyeE3loxXSEK60XTk+6GBtmP9HreK5Y4kZUKvtaLG1kxxk4b1MJXeVaJAQuoaIxRMY4lkrM0kWr3Lx5StwEvs9MK6mA0cVST/DQk8TLu2uMUcp1HVMrrJ2SSJvXlEKIxJh8gyxnGDhmTV+Vo6TmxXZW0LGLoiBuMnhYx6AGEOwcTx219iYMWQmMaITwsaDwUhg+RwCv3zTpB5+/MsiL5hX20POSQv5vDkuXGzFa2RtkHLjoRQnmw+hz7ojQlvHvSc141SkwMM5cE4Y6UWUQEocU5sUsJBCxdF8KAdPtOMUqlhYRc1gnrQtgMXLWak8MyW0nwNPF+6SLwK8oE2kAIQTQ01C28nPa/cS5iyUNEFcAD53eODhcYd9DHAj7DavG3FxhEImtDaO8C3CxDUaNWmY0A5M1hAj4M90TCm4XGgKJ0OucAYDIg0oVQAPYWeaNUfslDhyUItaMfyY1GNPP+pMFYt9mSDnhxrNuhaYzgWlqpwv6uE5iAjutbPH+Gjc7bSLyiyNATDSAo6XCzcfZc2C/ODok1N0LMzi5Nv1OB6OY2enprw3BaxQKJoal49AEoGBJYwciGLxPZxkqr+AGyNRMA7YRMxLdWjYQErXpSaIxYisGxcu8PtwgGKxKbTB6qGm0AJ4WBhUKQoRx8+IhQIsP4SIH59xLEbnNRk2hRMs6Nk1JXludHjDBNIp5Pt4T3EISH4grE2giBh8Pi9TKij3iWceSyg5TGVyMFnu7I57fz2qtJYgSdocTly+UEK5zLQl1bqF/nzI0A6GsBm5kDtcUF/CHWuYeAAInHCCFoa42a6MGNESFvQwzQwo/CAE6ULEh+N/20H8m/JAcro0CQRcGC83GqOxxU4Nr5XPKgH0JBCvx8WlL6A42Yl9kXjg89GX4c+2aJaIiMWmg8YF4hgopAzBNzc3R7loOYtyuIxXJ6zdSYYUNGooJm20OMp7M09uiKRsuzuIyk0QtMmksbOzbSEI4+uJsogYEcJFXB+OM7GD1Jce/aJsNrHtGj88HEjd5tMJup22EvrJYIB8sYRSqYzSxASq1UmUJ6Y8xKKDYyqf6pA340LRVlG1cuI6XebELbnP0IYTJKTO0Z7AfkfeKBGxXneESAkJC9za0TeaAJoMjr3bY5zqSBi/IoASU9nKjrmpUa7aKVAUXu7+yJ5xYiIk5ELyvzYA05m9rjhoy8vLyGWY5m3ImYpEBdOvBw7st3yBzBnnxeJ2vm9udlZ+TrNFUqUJI22tOZ4MpxjimQOby+cUVnEHVzwCoqqTQJaK0mB8z6WLF0zbFkpm5sjedSda8+Kw68hmf/mxLyX8ZaO+g067jmGvIyZIPmcTORx0iOojRQaGXPoicoUiKlML8gRJdqA0kiJEOHUwNFQqGCfaCV1yy7bk/Fy4cAGLiwvYs2ePecEOH9KeinjgryAdctdzh8euNrtkSX9OEAkKVOMUDl6P/zlew9oTQY8kSWSFtqVQKhSxtramu3CMAUhEJDCeOQo1zK9rq1c02advuwOf/Ohf49a73iCHs9M2XDoyf+F/MKdgmT9T54pcHCfgV+IOnLdxti43bbtlISIXmxrXHEFuImozmxyxiJIEa2uGIzBvwfmi3S+VLWFFTaJMpUgWBqumHvzS5xLyoNu1bQx6bXQb22g2ami36yCLI5fLmFpk4l057RQq1UkgW/IwKytUh7TeoiQsh3K5guGgj1azhYcffhhveet9MgecUE4+NYFiWIVK3EGkPNmDmUNkHjOFicTDRsPIhJxsqubAyvk3OljdbkdmCJ6WLOSpRSioxptmOElSgBZ0OJR65cQyAgmTwPtywng92UDPpIWD1WvXsLm5gTe+5W34o9/7EN7zDd+MhESO7Z0RHsAJDQHu9Q13N66bRR1yNDNmvgwhsx1Oc2eQr+EMNJvUKPSsFW45Pp9JG75BU8DfUROb+bHsXIZhpwSKiaqszKbRr90UfvTjf5Vk0n3UNtfQbzfQbTN+LYgmw1evb+nMtHO4h4yrBZ4QB88jTbJDvojiRAXF4gRKpYoGJL5VviDItdHpeVrTmBOBo9PmcMEIhHCSRdFxZC5if+4+Tg7NQLvbcWpSRfE3QyXa2Ga9qc9ZmJdCtcpkRV8U2vg9J4PcdArG1tamcHZOEjNh/EwQB8JciF3rW4mfbTS2UdvewA03344/+59/gG/51n+jzygJJC/egB7aawpKs1l/zZgsvcp8g6U9RcaUo2lzIoFwX4S7lbtaCaLQViOMwVk5bhKEySeGFWTyTEUXTJspbBsI8qVzq4TLX/zZf0u2tlfRqW9idqqCen1Hu6TXG2gnKF/NZEQkDpwJkmT5YMwDTyBfKiNXKCObLSCdLSKTy6BanRKVaXpyGps7dUPcFN7Q4zfHy0APc3I4mIhZd4n+fVQqEyIMcFE2tjZx9uxZLC0tKQ/Mscnm0oZlcyjm8zh27BiOHz+O6ekZdFpG/Y3EA2Nnzjb9kJ3ajpH0U4aARXjEcZjGsR3HCadz1GzsYGdzDdfdeCv++i/+DN/2r79LGiLoxeMevj1P1xiwYv0MtYvDJ1EWjQkPX/TAsoMsEk5faDja+OAO0P5qw4CgEfPvpEQXjXiS92oRYhTOy6P/QPuukPnDf/rBBANOWBubqysoTzhJYWjlJ5Q8euIcSHjc4chIEDI5qZpMtoBMlra7gHxxQna9Wp3GxOQCElJkCcP6i+GdqjGodpBCd2ATzAdReU82JwDlxZdewksvvYS1jTX9vecxcuzWcOzGVfHoHtz5JUYPBczPzOL06dO44/Y7BOoEZYcLFHbbgKTirsOWSrQjDB2DdnV9Yw2HT1yPhz57P97xvm82E0LOuUyMOUfhW9Cho8Mlm8xQivj5iPtmi8fn5e/DmVVenqZnQAEzDrrSlA6bCqyhqePadNoCkoQRgMCNcpNmNpywqSSVo2rSJb/xKz+eFLLMTfeRY/oysbonVmGYnbGgPC5CO0Q3n1IXjpI8cd0ASOdyUunZXBmV6iwW9h7FEAa+iKtFe0ywwGNvARwYKmy5cPkSnnnmGZw5c0YL0uoZm4NaRQ/ioVKABLHYoeqCIBDhEgkVfHCKFBedCRSmGMnEvOmmm6QFIg7ns0Y+X0BFwsXxWjKyaTZWsbp0Ea+756347D9+Cm++712iRtEfMNNjfLjIm9PTjjy9tJrnlhU1EATSHBAM4WLtEhW5Uw1MIQ/Acp00WSJe+m4NoCSfI9RMoqcnnpwzyKRPVI44XGj3+LX//P0JbVKxVECKnGXmdJkA8cUhmCV97xmeqMXiLjCuuZH7hCwxFOoPMTk5jUw6j/LUDKbnDmFyZlG5XQoMUbrI1jIuZCjz4osv4oXnn8dOoy5HLZIe8mYdirUFNI6a0Qu5YUzqRy/BmYwc7DchFBa3GzrHF8fBsIg7l/7I1NQ0bjx1CqdvuUVJlYjh47r83M72GlYvncPb3/3PcP+n78edb7pXBX6tesMWeWglReZMmXOpHcl/TvlSalh+gKlxIYb8zMDoTBEi8omocZjgiKcbkFYfxZBD80+4QfVMJC24phDsyhwFMQg3vYFmpn7xA9+TCIhPBihmWQJEN9/LdrSjzdBzNxIrV/VleIeUfDkkeaRdBXECaZyZCJia24NuUsSpW+6SNy4MmA816GNlZRVffvQrePXVV9Go1XVN2mYLxQzgtwW1laMW4WLzRS1iEmsPPVLd/n6S+cY/GzYw3isChvLmNE/GvEwPWVxYwVS1iltuuQWnTp0aZfc4ofXaOlYvnsPdb/46vPLyqzh2/U2y2TQtlrbkeI3kwBeflTl5YeacI3rVjoFHrK9lF2c9IyxD8XmAJq6OhRYWC2hRZauuwoTF5sTSzj4tUtkULoOxeyq62N3ZKaR+6QPflyhWywJDJh6YRRrS1hhFKQj7uyGRTbAyQp7jNpaG2fRR2pDFe4UK0vkqbr37rQIWRLYf9PHZBx/AU089iWa9MWJNWrxrFZ0Kl9xWxWLbw9kuEanPvW89rDMzYzEJqkilxxZ3Idjd2TZ2qVenKvNnyzkbIsg5IaBx04034fbbb8fO6hWsLl3AqZtvQa5YRaFcVdIj8TqrkTlIGS1bfgSdUa6E72gOWz7JWHgU8KuhjtSNxgW0/IFlBM2AkZJlSBsdM1HFXJOEuFui1lBN2/l0DFmk6MLxyz/3/oQDK5XzSDn91x6YWbCWFps7ke+PhAM/Ssg0dlxUUHCHh0dN9d5Psjh7cQXf9h3fJ/L9o08/g8cefwxXl68YgDJWSx1o2jh8GQscO9cEjjvbfIRQ7UNpZ+On0QSxIsScGtMMAlrGXiEUIUghWJaZM3iSU6a8fS6DifIEKqUK9i/M4NSNN+PW2+8UM1aOnlivu4wUwqaMDOhAEZMWS5Z2WaQI2wzyNZzRqw3j5BAurmWwGN6akFD70L5TG3EjjFBGpmhJn/Y5ZMREDSyOn7Sikys4D4Fs/uSP/9ukpKJwMk4oUgPk6FJ5WQztIyU0EhvipzG0cIaJr7iQLKnYtNVqK8eayeHVy1t45zf+n/jkpz+F8+cuaCe3O1TpVpyuHUYO1oi44EkT7TjPJXsFRnjd8uG1K6nGBhh4sZyx12yhtcjK8VqJsNlHI7jF38eFaFybjAtHwKb58gQI1jA+J4tmfmYex6+5BtccPmDeL3qkfouuJIFNzLHV7vTiwVjgKPYzgQzv2ahFgmY7lsAJuJNzTY89dr9COdaBZ4NGxXsa8ZGOXEC8xrBJI0XYlvyBX//Vn0zajQYmq+Sb9QxtoipKvG56wNJQBu4GBngkotooedJEZ+QtkqFhD6b0Jx2GXBk7/RKefv5ZrG1uIDUw4iCxbNpk2maFcz7rsYBhm2PhQtWG6chI4o0LpyyYCmK4iJT0XY41d7+WX3YuhVTGhGfcnsf3sdvHfYBIJ3Lxc1TtBZL3c0bu4KISfi2X5eFP5LK47fQNmJmwShBqiBFU6hUZdLgshbtrPhgDBz4fwEqMyWrJrALGVLz5TwRvbOGNI9DvGRaiOfDUcrBc+DMxc23WD/3mB5LN7XVMVSYsC6UkeQqH9h/Bvn17MDU1o52aLVWMJeElran00PK+nabiPe5WOhgE8pP+EINCFc+/chYvv/yyUpO0J60mHTDzsBV6yNu23Rn2OB6Uv1eO2RhyI0+aP4loPyq8J2Y8MJanY+KBfAnpc7LguJMW34f61jXdU9+140b0I0TJF/EDZIj/M+WbR67AxFBJDpbsvfyeDMrFKrKpIfbNVnDztddKEzDC6QtYoa9jzQqIVyszSIoVee6OM3Ac0nhjPooVRXhRorho1q4EKdvhUTYdqePYHBIW2vVg5Xz6H/4k6XaZ5aIt6WN1dVWkAuKvlCLaHbryzIpJUl18xIPOpOTFmlonamRgQJLL4eJmGy+9+KKcLg6e3mGzaYjPSK0ZlVrvsV1kYU+kN7ngI+ryWDWE/C7PiZvN4mJzZB5aOcGBJsfE3VKioSliYcMsjNvzEDZG/0aiMEdIi6SEQxHFUkVZQC4UVaS0U8YBGAqiV8jksmkUc1nMVSq45aaTgobTXpJLZyvoybLPo1IdY+2qqsRLltR1watCtEPdQeYGi9DLtoQ5hTJhgp4jXrcwL/UXf/RLSqdQCsx+GrbLeqSwlLcAACAASURBVGVKEFWFpQB366t5MzpYVD9cSEuRplApl5CvLqJXrOCVl7+K7Z1tT/dZxobCwCR/qGsuWDgY8RASHKFK9PAt8xYPZ7nrFLIeUlAABfprt7CyMoMBQ5mITp1HF5LOz47b43FPPDJc4dD1B8zpm2PFCSSOzs8TFqbJylcqUum5gvVqSWjC+kaUVIHgwHqqsFxI8zrsygGeLGXx7ne8HSxl5D1VvizqtFWrBpUrtJIxTswkBMxqxY6SeOcAmh/i0qy/8dmiPs1dFqR+4xd+ILHuOlbiQlBBXQdy5FSToGDeLKmzQqpUOG/0YpHbvc0EXaFBfhKl/dfiqYc/j3q7hW6LjpgJCz9HDjZBei6MFtE5zrHrAgkL7jYHH4BNCIF2WYQXopsx+LTnlKOUIZ7kxQgeesX1YyG/NpwLTRM73cIWCwNDy1CdcxMYPFxEkiNzp4wkYzufQsD38FqCdj3lmvI0roiVFM52C1tXL+H2G6/DO9/5Ts/W2diJZ/Mlb97JFRKUsZKrCKtIkmDVjsHYHoV4XxjLqRv3PIAcRQS/9cs/rG1n5D9ic27nvPoiiuRMzbgO99KfiANbrR0MhxnsP/12/N3f/SUyDnZQOxiNyJiTzDoZB4w/m80Sb83VdYRtob7DBsm++w4Zt62pUH9qCUVfg8O3/HHs4PAFIqQLJ2/cRxjH2GMMDKG0WxyNE1qo3LLVUTHTx8RPJl9Chg4se9Kwhj2VQb1hiR9OGGu4FF4hjXTSQ7NeR7u2iU5tE//ym78JJ48ftbptItxO+DAGi5mRICMGrs4oRxx4gkwwGFUl6iRDiMpkcxuVNJFdUzLlv37wP2ixVZfsZD05JE67FewmgMOACM5vgP02EH4uwczR2/DYc1/F6tIr9neVsUTLJ7NrDCcaDcKmJDdSEMx+M24OdR12VWqIVZNy4v7/VYzane5lWu2MIUtc7FDX4Wz972x0/C7s9bizpmuz84SXB+k6LlhRCWI8vDzSuRISpRfJiSvK8TThNAezXGE+voE+bWmvo2Cwtn4VrfqWHLef+g8/aowez9eP8geROxBl2KBYsW2UhevLUMlNUbxOyNXyF7wW7z1OqwoMI/WhX/mhJBZUgIX3BIv6qmBXWALe0pPuH5tXyf+dFvLH34L7P/a3SIYNDZxMC8F3TMnxMwJDDPK02m4Lk0wN79rmcFSsPHfXWePYYkxRQWnjME63TJbHcKGmww+I3bp7bbNv8dz83jJ4RpDQriSvzZEv+QxU105CMNvpoU62YOYuV0A6V0QhVxSIwQVniljz0++jTnIGG24NE2ytLmN7ZxXpwRA/+1M/6R0d6MgydUmVbpskiBARchl2bhiZxeduucliCQfWKckjs0aNOCTjN4/Ub/3iv08YQrCaIfhhu2GPYa8RAoUDZ5JvO55aodnroDZ5E557+CHUayvyUoOcR+FhJ0LtdudHEVMW0N8xcgFDMKk6955t4i15Eeo7FkEL57zvWLyAH9NZW0Q5bWMtu8a97XD2wqEZQZtj8Kny7EwFEqgcYdVWshTqn0V0NqHuw5C/njMiZrqQQy5rxREZr4ztscojGQgf315dRr2xjnwqg//4Yz/ila1dLSQXJgoNZJfFErW+K9FKLNp1EBs3pMyRNufnGZpsXj2/mgYGUh/8T9+nKk5WPoSBskm3zJDZM8szx1dzZAylYrhEqtLmxLV49itfRLOxpsExqWDCYzsyYL4g9wVRn5+ntgjnKHZbnoUEASOSOapWGUZb4kv23MEVLTpBBu4cx8/HwZH4Pr4K2Bgj/MeCh6NmKt18F4Ieso8Ou45/TuPwWD6XLig0Yx6/n5D4UGLnS5RLJEZah0JmyQrZNDZXCRevo5jJ4Sd++AcdLbPuipayNAdTIIwDMOGoKUHkfsS4mQptFlrMwBbWirtW5dxxsWUPnPX5tZ5qEP/dr3fyn4Hz2o3suNDpY/KGd+Lxzz+AixdeRNY9VO5wMk0M6SJD1CoUgjhnHja9cgM1DB40ocupoJBCZa42Q6qAT0cPOQb6K+4nNjDWqoPPFQscKjoctPHnDOctBM5UqAmVFbfbDhnVTHmZrqIRvx93eIoOWybHDJChXKRZFyc1hiafvdVGIZfG9toyavUNlHJ5/NSP/ahrNIIO1Epm7zkHyi94nbnh6bYfd5MlZsi4uagNhNx5HkB22pHMqC9P/ebPvz/hgKluwhGKna3p9fAodpOBdmzlZIxKJgJanT5Ofv2343P/9ABeefZRZNJUw6wVtvJdAhGhsg0T52TKuzDKMLsVhN11hEwqyEOvcDYi2c8HkkMXjXr4wKL5WLw5WgDPzH2tGh/f9eO7elfr2K6WgIAolJVARdGinM+BJzBYo6XSHysglLOWNgHJ5stC3bhjudDKQPXbqG2to1nbUi79R37g+1+jrYLepDVx51g5ctcsMUYrLdrtLxsmRqGqGEAUxF1QSprhN37ue9VAx+LBcFJMYsxT3m2foR3mHYXDzhK9ajVauO6d34Gnn3gWzz/xJXQ77NhgHuHkpBXDGxZuVRoR+1kmJ6V8dixQ5K3lhHmMKiKe57HNSfOiAW8UQGecjk/kt83W72a75FX/bwraQ+XLprmDE9/H5JFLxvdxh4emkJD3jDOnZxqShWPv0SKl89o8SOeQVTtN443xvflsVqyXTquOublZfO93faelI51PF4Idv4tx8e/jYwuTE8JhPpDVltNB5L2ClxDzl/qVD/w7lexavbEjVGNNVqN6kQ8RN+CFFhYWwBYQxWIeSSaHzuQJnLu8ise/8KAexpy6IeYXZ71wwOyWhVKmqqimVNM84lPvdn+IQgOOje0raYMCD4/sFheedj0ctkhphoqORY5F3Q0jvZPDGGWY4+JzRQgY6jBaXkdnhQA4ct5zRmgZm+8RIVSM7w1o046sSWPSnzVGSqrLxj/b4udff/11+OEf/EFfbGO2hJNq/lHAqJ5p9HZlaTmHDDONYxa1cdS6mltH56h9ogpUc/BLP/OdymczbolYkzsnVGXknMnbYq8RPvSo1ssTCCwZquX24NIO8MTnP4Mrly+OgILyBInwjEENFQpEzXZL3hrTpq2nWBD+xu1sOGJmUkIhW2Jf2ACT/DExY4iZdp+XvgYuEJM5vtPDHkc0EL5DaAIrKjRGy8jR89BHvVy8dZeySwlZKabOuU4K1cQxy6g0R/dXjqAuuPRd73o3/vk3vHdMjTMnb+2/FPJGaOpOqXnf5mkr7aww2Xh9Rllwe27fjHiC8WypX/zpf5swSJeKYTG351S5uATuc85bjpCF8bEe2u1jmlNNzzFVwvnuNB556LO48NWXkMomyInUDiwszo2AFAvx0t5vu6ydHdpDu9ix8NiNoY7DpBAXd1/JAIxUImGx1N5uY55Q5fE1JinEJa7Pn2PXCuN3vH40qeS5ec45FtxqoS29Glg2+WEquqcL7tGCqWAjTrCXaTTwEVU6ncKHPvQhlUiHmRPbhw7pWBp2V0CtBp73NQ3rFC0nMHCiJdzeL2a0+B45aSwf+In/OyFXiv27SbpXB6IRMS9tOLSyLN7wLpIQUYutBu9ZdIcJznXm8ORXHsa5l55Ft99GOrHWUlNTE1LZFDcurrzMPqE9a0jL3msGtJiHHwAHB8hdoqY3rE5UV0Dz3G3X7qpxg3stsRI7OhY6zAavN55wGXfUYnF31WhMqoFIRtm1/IBSvS41I+dJZLY0uh0nGoYdbvdUkkP1ru5L0XigVMQHP/hBoYCGVnr1ihMTuKjGOHGKkYeD+tmTM0ZiMAatSIteVGkIk7FUhcwpu5hC6o9/9/9J1HzVS2eEgdDekBJM58JPGMhmmOVJI3EUiQsshIv9vAg2II2vrnbxwvPP4qlHviSCvvBqVmeW2LzVPPKYVLOPhhoV8+wRYrxyld96OBOLEwLAWnH+jTtZsbtHBru7w9E9j+3Gw6zxRRy/7tdqgLh3CA0xcj4rd4xahgRI4YsgJ4222Om84deElookje1QFjQaF+/EyWvwH37sx91OBxXZulOpfwrDWmbt1FLL1HIIp1KqhRyGHWeiOOql4zjU9M+aBFohgiGRCls/9td/mBTLRWTUSwQCBZKEKTfr2zGi73oFQ3qw60QpNEmxwRtj3DSu1od48atn8ehDD2B1ZWmUiy6W8ihPGJPFvHEvuAtb64sbPkOYknEHSw/oD0xvM4SGYyTGzOvGZHxtDB3OllKKXgfN7yMBIgFyGz+uBew6VuhOSFRC5zy34I0x2aNIIW190MI+mgOaRTIIO2u5ezstIY1f//VfwczU9AhsspbfFs4JKQvbzHvGbg/AhbaakYznrpW/GrP1u2RM3ziujVMPff5+IX9q0KL2y757vGwm3H2Lei0nPY4hy6HxdFo/yeHxVy7jSw/8Iy6++qKpmEwa+VxWhQfRp4XccF5OdUjFDLpt6xca6pkTHs1aaU85iVTz47tw3KabJTPHJUKRWPiv1RKx2/lc4/cct7OKSZ0gEOxPYeXBb1NDH2eQuhYZjzLsnhmFWeY505QbCklG7Xd/93fjDW94nXPw9FcRMGge4h7RrYmXFzVpnA3rfPQe07DUKS64chIpcKo5G8rsGcnRk1kPP/JgQk/R0pykYxqYMALhnWLbb1uXWz6keeNx8k5KD8JS3VyuhOcuruIrX3wQLz39+AgUoNQyfjS8mXnznpAhkeDTAyR9CxnGqzPi4aJOy0AZE7RQw5EsYYO+r0XG4vOhHcIPCDX7tSp+3L6H4IzfS8wVz+Pzmv2ehakhMCEs0cFR3HkdTZHHgYMH8KZ77sGdd95h+RWRRUwTRe6BZkkOn0cQ0UslFt9Ewtil9PLDWbOMJVG0XWbqeMtt81E8qfT5z9+fsBMv7aHVPRmfigNSAl0XIqmcRXQseLOeXqxgZH5a2DbhTZ2pUcCVtW18+nOfw/NPPKLUpXUpsm75LMfhBLJVRKdjvcJZE8XidoUT8jDNQYtJCE95F3TZ7T8mQqEcOscH8plRV4TAv3fBEXOc+IpESahsmYgxtC3MQGiPuHcsfpiC2P1a9HYfe/fuxfu///2iHhsM5Pdy+rAEMG3PZxTh3TGxr7uIEuwU6Y3reV+WRRlgYk2AeS91qnAiYtC2rJWJbRoCQcIlIivorcVSD372kwmzVjqRJ2vdh1l7FQDEoGt4axSuST2pgsT7blLd+SEtjDFT6QKefOUM7v/E36Fe2xoxIwnAWO/SrOq2u11SZ62WizaXLzEyHXCJiYoJjh0+PtFy1EZJGh65YDZzHIXiIkZIFRBo7HK+N8xULGjYXA1ojIgYAjCeJ45dd8cdd+DffNu3e67AKjZpQ6PG21SpF+2JXGmYugmZVW8QhwgnkjtcvD0nDHLhtHO9k4L5GAyTdxeVi22JKzp0Rhahn0EBoGoX+vfpf/ibJM3QqdPWLstn85icncYLzz6FYcIwjJBnFXv37ZHtaNU3MUgySGVYrZlHZgDkK2wIYwxPqphXlrfw9x/9G6wuLwlDZ5E4ww+q6Xqt7g3r2BfNeoMOKInOlFEI70kRIy8ECXG3VktxtZzH6LliNnZ0ksAYOTGw5JjIWAC+N6jIdoSUYf29riF8/G9CbdpGCQ5f/NAEHCfr2n7mJ39KY2ZhgHqjD/qqTbfEhqVbWYynpvYD48rzFa1GuLBEIlUbzoZ9Y3kBnVDk7SrDbBCNMzqxaYg0mUHhs+ikBeMPcvz0j4zFk0Lqr/78D5Lq9Ax63bYkgdX611x7Eg/d/wkcP3EKi/sO4+WXX0Q+m8aBw0fx8tOP4/ipm3DxygomJyZw6dXnkJ+YQc/JJCwiT+XzuLzVwSMPfUYdE4kzVCtV84QdoCB0yvBASJDiCqtdGn+Zat/9XahNBXoKKSJDZHlmkiNjUUMtj9vmXe+eMazVnekeHpoY08N7sPjC8prjsWqo0sgw/b8/87OYqU6pw7HUvldi8Hk4FoavfFajEVGT2PtCg9gzMS9hVCRRmdzzj0NtKDChUaTxmPpVBMDuzz2rvuUpB+xVquY6lofv+r34GYFVH/nw/0hm5mbVe2t6egoXzp3DnXe/Dl/8p0+qo++RU7dgmcXvVy/h+tN34IXnnsDJ625Coz3EwsIcHn3gozhx+s0oqEVFHfv278fTX7of5cM34S8+/GEsXVpCPp9RO6geC/ac6cLJ4aFkQnpiQcc93rGFJl4VvTsNVCHQE0wWS4wYkGKCQVNjDppXcnqXYOamJQyBKbN6xc/90G7lzus6Bz1Sq9EiOrEMHR1F64OSYHJqGj/3sz+npEh446ERgnI1KgOWX8IerB3tYIJNpkms0Q0PYlPNupMuIoyjsLIxACneuXzBKkM8VCQMbfQuo25Rm/R40kGpKN+l06xbXThbpdCGs/PC3MI8dra3MT+/gLOvfhU3n74Vzz/5KNqNbVx7+xsx7PZx5sUnceTkDUpyFEtVzC4eQnlyAk9+7mOYmN2L/Ueu02IfO3YUjz7wcUzuO4LOsICP/t1HUaMq8dZV9DKFJMkeGUU2asis04QdTmbVIl5HNebIjHunEarJ3ku1pcSQMTVoFY2aPDXX3c1ta4d7VYWS+4RMM1YjxYlnSMjvdz16i5F5P3rXFk7mVaX5rne+Gwf37hsldsLBJFeNY1LbixZPTjCba9i4naQQfk803+NX7sDwJaiGubhsTBC+C7/yOjqZIA1t0si9B6N0e3vHyCNk/uq4Spbx9pD664/8fjIzO6u2FWxNwSTG8ZPX4crFC1i7/CoOXH8bFucW8NzjX0B5eg6TlUnUG01cc/I00rkMnvvypzTA46ffpAXau/8AXnziATRrNRw59UbMLsxic2MLTz76EL789BksXb6sXWGevrMynMkSB4lG191oWZl4q0h+jhQqPgiPfeAujxYUVu/sPcZGoIsd8Cq1SJUfdc1OiJQqde+fAIXh60Md+CoMWiR9o/bypTiYcbP4vEAubQ1riO2Hz3H06FHccMONygqye1TUG/EZFNuzOW+vp13ISwVMSgRRi+LnpfCrteMsqgcMhZj1d1w0CZu34OTOpkIzSDnB7MysasXYnSoO4su62Uj99V/+j4TF6LWdOqqTVaxeXcbhoyewvbmGK2efw+yBa3H0+LV48ckvoj8E9u87iq3aNvYdOI7iRBlfffJzaOxs4/ANd6HEHT87iwuvPouNy69i7vAp7D98rR7wxScfwKByAB/72Mdw+fKyqb2BdTgO+0Xpj7CEoQapwnzIyLZx8Ny1Ukm0/Q5YyJN2gbFsmLXVjOI4LZYxHV6T16ZajyTQbjLFD5rLG7NVbBSP7y0c9DCR2kQcNW8G7zn3cNCII3CcLHZg/7SJsp1lwrCM5nHYbSmKoa9jdKs0+sMu7Y4EgYe55Qs2N9T/1g/V6r7Y+ULOGokjjZqKKNVpiTVfbPbXrKPJDlM6Xbfgba0HSP35n/5uwqpEa59cBM+Xmp1flId86ZXnUJpawPEbbsH5l55Rw/mFPYfEpZqc2YuFxUWce/ExbK1cxsTiMezZd1iLvXzxPNYvP4t0YQLX3vI2dSB89bkvoNnq4vMvLeP5xx8fqR9BmNHPVOwV271c5JKfFMDfaZFzu0kaIWV+Qq86D3i2R4APTxQKh8lLYwngMOHCtKrRjiyhEWaBqcoAddQtSr3COXF2hgfbVZl9NB+DZT8sMOQiqZuTzibxhgEOdFBQeF/ZVPfCC/kSDh44iONH9mNl+SoOHTupnnArK1dRmShhdfmiHK3DR67BytUVnXaYKxZVhdlt1sVJLzAbmStg2GubZnNIt1CqamytTgvVShkNP6lPWolz9Vd/9jtJvkxyoDVutzjVmrGtXDwnZujJG2/F8tIFbK0sY2ZxrwSjOr2gU/GuXjqLnaUzQLGKhYPXYnZ2Adubq1h69REMBykcOf1mdUQ899LjaO9sYjs7j4985K9Q11FN5pUyZOFXWtp9+/Yr3hYzxI8nZlTGn6lo1ZMz2l97VaaFFlSnFk7xWlJvcaY2QaOx46oihqeaFN3XF5+2UPdxhzHUvFKq7jCypo0aYZzUEeDLOFizGzNb7xQV5jmGoNjeyZgEnt56772YmpyS8DY2LmNicg7XnLwJly+fxc76KvYcPIyt1VVkEx4ydxUz+49jbn4R68vn0ajtoFouQIfjFLhBymh3Gug0a+i1TdAIdnE+Un/xJ/8lId+Z+LUC+X5f9pDhQH19BcNUGvsOn1B/tPUrl5EpltUMNpUpYe/ePdhYX8ba2efFtZo7eB0W9hzAsN/Buee/qCMo9p28HYcOn8CVSy9j+/IZJOVF/PnH78eFM+fQ7Rnezfvu3bcfh09ci/m5eeRy1sEvuv30O9bnrMQDYZx2LBXrP3Px5HQZqXrk8Qu8oPCy+I5xrjea5zPy89FFOECX8URKNKoNgYmkCSnBStHGkY9RPDiWw+Z4IlY3xGs3JByhdrLhPF/T4F8ybCmQxw7OYX7vIdz9unuwvrKEKxfPYe+hw6htbKDb3NKc7T16E0rVKVw5/zLQazGzquKLfGUGM/OL2NlclZlg10rejzSpEos1//T3fzkR31nF3XYqnzrRF/LoNJuC6fbsPyJbsaZMFoeWRbZYxsL8HkFzK+eeV0gxufcYFvcfE3l96dXHsbO5ganFAzh6/BbU6ptYeuUZtb185lIT93/606jvbKDR6eOHfuKnUW8P0B9aX/B+t62meYwfCXiwebwWiIiR0CnGqhazdhjX09apM7E1j+VxVRFeqcpFaUMrciAwRE1g6VaDaMPTDR5XcMnioNnIkAmNU7WqMWIDsKHNpcPJ8NLOFfXTdrx8KFp18/ddnnnqfcfl7XtmXGeSqZdMTxSmQwcP4Z7X3Yna5oaAm15vRwvOse+95laZ3NrmEmqbV9H1as7yzF6kszwQponWzgpSgz62eYpvZRKTc3uQ+uPf+/kknS2gQM/RWQ18eC5Kp832WAkmpxcUpNNpo//KTZUrTmDf3gMCA66cfQHDfhPpyjwOHL4OxXwJaxdfwtrVcyhOT+PaU2/ULl8+/6zUYbtyBL/727+NlbU1fNcP/LjKaLa260ilzYwQwKF3WSa/LUlEqqCw8RpimGZJY2L/MaYQ+xh2efRCH722N9cbU8uWGrXr2kIbYNwmsqdG+EaJChiWX62Az1pYRIYvgI02QxgnSQaiJWqSw7KMcdXbTYV90aXJEiZ23rbF/vZ9HMhqHRSkPVRTwTH1UC0V8N6vvw95HajXQnNnW4zUvcdulTlbXzmP+tZVdFtNadvS9B6Z1+3NDaBXw9ryZWvik6RQnV1E6g9/62cSNpnLuo1MeUaF8KBaMOoQlylkeUh3r42GmCZZtdCYmJyRyqfdbuysI5cvYe/hU4JXV69exOblV8XeYAjGU9uvnHse9Z1VzB64Dn/2N5/EiVM3Y3pxn45n1IEvLEFVKGPg/wghEzrURSGbt3M1szxkhXGmgShpgjE89LxnXYLZs7TXZN6YkGRXNdGKad37p9dPDRKN9tSvLE+wYjCCcFlxysW26CCl7gahBfg7zoslM6xsmDvbnD5r6MfFEA7gvcKjC4Oa0PF0AF7DY2p+r2ILfc5r5HrWFLA6kcc3vOPt6LcaGPa7SJcncOyaWzBIp7B+5Ry2rlxgcY5M4fzB61EqTmCYdFDbWMba1SWFqRSwyvQCUn/wwf+YkKhAiaItYvsIhhNsXqf2Dil6x1UZeXYopoqU9BdLKFen5KVurS+hV6/JBMzuP475hUX1DVu/8JIWYM+J27G4cABXzjyPVnML5YlpPLvcRXlmDp2etd8S89QXkhk224l+aqA7TMzMyXazl6p77oasWSUoEyqceDaHS3kbCi4YPVnZzYT/DeumqdFB65HedWKAWlzJy/YjLbwgYChTMlCOOrSAOYK77BtpAbD7RFvevPkJ1pGY17TkhrUXCdqQBMd9iPBfDDJmVScPaAW+5Rvfi/SgZ+ZtagYHDl6PHoZYv3IejbUr6LGWPJNBdeGYmgT3ei1sXL2IAR01xuoTFZSn5pD6g1/70YROGNtIkFrERVZK06sp1JvDKx0M+7W0W5LKYnJ6CplcEd1WDTsbqzqFoDp/AAcOHlEP1NXzz7PfFqb2X4vZvfuxvXYVm8vn1PZyYt9NuLTdwOb6ttAuJUl27LhFmgp77Ta5s7DL6sO5s4lghSMU5bWMyyWILhQcL71QCpESFd6ey0piTCtQGFhTpSMn/WgK4eXMoHmKUhAoETcJgZU80RsPx5Dawzh1LHw0UkR49LxnOHcBgYawBFrGnyk00gxjPVzlHWWzeM+9b0C1lLPqmvwk9h44KlOyevkVNLau2rNkM6jOHQZDO4ZrO5uX0anXrCd8Lo+JyWmk/tsvfH/CKgZCRTlWIFKUrNLLzqygM5GyKkURERkzisGWQ5GdFgoTGPSaaNW20Go0QCeBi02MdvX8CwoBJhaO4NCx42g2a1i9+AobV6By4HpcqvWwvr5lZaaqELWJ4iIrJednafG+ERLxIQmSiEbknCum9Pi5qNfm7jOWqhMTiaDpyGg7tkH88yGUk9fnlIywMLA7sG4S2ZQVshMjUNJDXYzICvW0qHvhhoFbXpq7qOskD2kYp2AFeV+dFb6mTCcSKiGMwaAJX4Ff3/2W12P/4qzWZXrxKKbmFiVcq5dfRae2au23CnlMzh9BuWTtvzdWz4JUETmZ6Swq0zNIfeg/fXcigqHjyAmbzbK7AltLyzYzCc4qA3c2VFCQIJPn+ZhF2XpOXmN7045xqlaxsO+ornHlwsvoNtaQKc7iwPEbJCjrV86i3+mjtHgMm/2iuFRXr1wxRMhPD7BeXl0hZOEpR1ZMRx555YUQLSpELz5Uk9eoBGU9eJ4q11RmxOKWnuTCkCnCyfDzNpyDprM0WJbkvdA73ThegpSfFnLUbqQww05D4PUUQXS6fta3lSSHLQ8nLnZ34O2RJo0jKFyVuYDasVFxxOV77nsD9sxO6muDMwAAIABJREFUSkUX5w5g3+IBLeLm1bOobSxZGXRviPk9R1GZmsH21ibQ21I0pANwGx39PvVbP/sd1AFyoDgwNokXu8MdDJaeplM5JDnLVVN9m9NCmnAJ7A+mZCNVx9YWUrk8Fg8eEzy4fPEVNLeuIElP4NgN7kEunUW31UV25iBa2WnVSa0sL2uRGA9zt6lGKTPEsD806JBN5ssT4IlEskHecC8otOwWQc+a0Kd2ijxj8uDN+7bOidYWK5L+dK7YYpMTpaSHs2aiSWyUNxGv5vENwx6dKPY86arUNpoXtPtdMw/eKIj4dajigIEjPx8xdhAX6DyFoxhCbQ1sR2WaEuy3vek2LXapNIGpfddgbnpBuYzNlbMYtLcUmRQmJjE1sx/FiSo67SZWll5B3rVVNlfEgIWHH/rAdyZiOaQtO5RmGwmiUZ6xIQKsGmVWJqZTVmzOXaiOPEWUJspuuwaob22LZTo9u4Dq3CK21y6jvrksFHnx0CmUKhWsXTmPZn0HufIc2qX9SkRs7WwpyU71yyOQAokKtRyn+ubyhosTdaKNJVOTqUL5QGOlM2Ez6UOojIZwqx+uqkn1BjTMGFEzWJ8XClZeuLLial88xqqETOkEqTmfU5iUVnXnyrxpO4SdziCzXJEAEVbujFad3R1HZYjM4Od8e8M6TmQc16gx+CE0//xdb0KF53snKew7dBIL83sl1Mvnn0ONNps59HQWE7P7VRde21lDNunIBxLUW5kStzD1X372OxOzOVb0zZBLaFTBHDX2CleaMLFQQkcTqNk5Y/Gy7IF1sx+q9zYHWChXMLfvIHrNbaxcflU2ZfHIDZiZWcT2+pL6irAJfXfqGvkKXGweDcFqTsbtUaHoLbSlVjmZhFE5JmLcUc9katGQNf7nwgX9iMQJ29nBJPXKEYV5u6fvMU896HfkeCrP7nGwbDeb1PJ0wFJeKBfrzsLDVt83liA7kKJkhjtYTGTQOYquhMYPYzLeqFfRwcJy7pGPtwaC8iGcEcr+qd/yjW9DliatWMb8PvO4eZrP1sqrqG+tWPuNdA5z+46qgrTZ2EK7tqbjP3QC4YB14hWkfutnvt11hpXQBhtEh6MzvFExALnZWaTzVn8sJiSTD7Tn5K3xZKC8nYqrcy1KE5if36sdtXb5FbFVJvccxszcgjr4s3mMSIvlEwpVOmxDUa/LuYlcbuDVlvWx8ETd/dkf1Q84CcZKwkXgJDsi1uq27TQgr57kLlVhuoTaGTHe2sPOv+buMz67cs6eCrW4Oiv8nCRJOX19rzrReR5RgUJBs8pSMkeiEQl3KtOl7CYch89F01i69jI3znc3X4MttqzDAgWHWmeyMoH3vO1OTFan0RoMcejoKVQmJrFT28L60lfR7zYFnKTSZWlT9UEb9pB0G1hauiRNUixPYDhII/WbP/2vTY37ohqldRdW1NmWKo/M0OCpFFUYsnho1geMks42URaCMITIozI5h8rkJJbOP492s4nKwkHMzC5qR+6sLVviYvpa9NgxMWV8rJ4X64fHysmXSiY1iBAn04I6e9MSGNwd3Fl0jnhdlsFGaSwFNc77oAqLuF2qUud/GeOFcTX/RuFmbRuJAqq58lBqBIl6fM2TiMPmmrnY7aYcp/Ba41w3LXQO++yVZJTrqLSMggdreGMLLSrx6IjqtDTD1FQV/8c736S5nZxbxNTsfoVXPDu7sXEJnXZNglyd2oPK7KLYNIxqCKrwpGSmr3fqdZRLk9zZ36Fi/MjcREDPiVD44+CCtX5iC1s/c1pnhDA+ZjuJtJrCMUHP9BxDNoIwk/ML2GKXgc01ZAtF7D10UiqPP7MNZmX/ddjqG57MhHuj6Uc9DW0RR6GKdiorTzpIuEu7hpUTEVP7KLbS9J7oXLxI6PBZomCdpkjtuHg3jdvqrWk+goIbTQLkoHq7jvGwyey9dX7UGVrcJN4dOUgQ/MoIYLz/anjaUZAoCpXrU+5sgwGN2B9IG1uAc17vufs0juxbtM2RLePwsetFaNje2cTm1XPotWqoN9uYXdiPdHZCm6DXb2NjdUmhqDUw4Jrlkfq1n/y/VJ8ttTFWlmq4MGucrMsfU53y1kX5zWHo3QJ1oEqprF1ON39re0tYNosGipOzysisLZ1DtlDC/P6junnS62Fnex2Ti4exmSygM+Ahbzy1hhMPdFpNLabSrCsrQsbUUbHfwvbahtSikKiehU089ti47XZS4Hi1pdGS/MSByIJleaotbbkVHhi4stulwPhscYCLV0+6lpFH7WQ/2d047H3sFEE7etF4YSE0VmCw26dVrFvaZTpq6pC4W8BHLcCzWk7fcho3nziMTqsmBK5QncUij+FImGhpY3PlPHrNGjvJoDqziInKnO7RaO6g19rRQQHUVKRIsX9b6hd+9F8RNbbzPoTC++GnnguWeo/KSTVbpUfMHizehsIPbGOF8GR1Uk1pq1PTlldOpTAzN4+rF8+jN+xg76HrpHImiadfWcLk7CLWM3tF9WFMScePue0aKTU6M2tTCRFmgsjk5RENje0dqXvBlElw2g1vHq9uDApSLLx2ZZza5+UycVipOh6JyMIODFGf6ScI+yLuxskegqrbgrFbuctD3ZN9kuJCC//uW6/vsb7qTGqIaDFioBikGqzVfDaDt977Nhw5ehS5BNjavKjsI9X9/IETmJyeQ2o4lBrfuHpOY6YWzZd4tGNFgkuKdrOxiWG3Y4fJcjMih9Sbbj2U3H76JuxZnEW5wGMgbGcYsmTHOUnL+JlVVNuSfB4xIftt8CV42MpE2equqxXtNDam3X/oEFaXltDpt7D/AFG0JiqTU9hcX0OhmMdw6jp0kBOjIzhZdNSIVtG2Moxpt5totWroNNtqkcm/G1drt8JDp+xSCBMoHAv4MXaptFLWIFYdqRB9x7UQdppwf2AkiqhBD7ttTiNtOyfDW2RFoTyv56Wz0jKEPcWMTsk5ox7ghomW21UeLyV2ib2OHz2Kd73rnTrakX7H8089La0wOTcrz7+2eRk7W5tqaLD/6CkU6FUnJG3WsL58Fjwsjru2VJkBUkZy5GIPBy0Mve1GVwfDVZC65YYDyc52DZ1uH3vnp7BvYdKci2Qg7teeuTmxKKpVghpMORpRwFgtwqasFbPjuJwoeucKHZIheEYlJW91dQULe/ag3e6iPDktQiL9vurCYaxiHgl3sLJUHaUtZZO7jFlbaDUbqO1s6G+M5UmOCOyZE0Shi1NpFaOn2bynjEabJTNZxc/WoZ+JClOlPG6AgsoiCNavjRIgsJpoU+27rUWCjCDVOxiiFGd48z00H96TLCNUz2JrhWR+AnAqm0elmMVEtYiDC3tx/fU36Pip8ClUxpMCnnj0EQlloVpFv9XC1tplgGeDF4ooLxwWKbRR20aztYN2bUtzRH8qW6yiVK7aCcHtJrrtJhKCQATApE2ySH3vv7o3YTqvR8eDXYa9+ZyqCr0/mb7qRAErLdGBLf2hFnl6ahJ79u7RQSqGaLGSgtUQrGe2Qv04TqJa5Yl5fRQqVSFOxL6LE5PoVo+h1UuBNWeKibsdLQ4dL8boGxtrGrg87xbP/zLcOcJEqWOPkYm4EeUSEZD1awXrrM+QjQfAqgyHKFjBCIUsT2ZhgEgDNGEeOAU3OxbZ4E1r0MvPTfL0PyJnLhhWnsPr28HqFMZKtYo98wuyvRN54hCb6LR64gIUJmZxww03jLo+EKmjKfvyF76AieokSpOTWuy15fNqbstoZ/bQtfrabtaxvrGiEJbRMdkz1akF7XpD69qq8GFYxnFIjdP3+vkf+iZtEjZmV6rNCXW0wZwk4b7qprRbtald5z1MlaPyqg4V+fnpPTOzM7j2uuvEqCAIYIOwDj4E7SNVqQashTkkU0f1WcbqFBR+JQOD8XOzuY1+u6OfyaYUB9pP9RXgIgDD2leJBOAn7vCe6YxVTPa7BF94CkBJlaOBgKnvJ59HqVbadfNfmC3Ty7NbnFUlJzy2Vh8G92tYp8Wdye4Kx48dU/NZ1p2RYXLoyDVoNxs498LjSPptEGsvTC6iNDGtkwXjUHoWPfL5udiV6pTCrPWVZdRWz9uclWew9+Bx45HvbIrlQ4iaY2r3eiiXp1Am7yCblT3vd5mOrqtdds6Zralf+YlvVehFhUz4Ubli5oVVAdGjhTJnw20UmV4CKFxN8fd2Gp1liSIG5c6k/TLbbwT9bsfO/5pfXJQ22L9/vzx3kh6Ge06LVkumZiQSqKLIrWq0ttDheZs847vZsF2tQ8GNzMAXcXsKJl+BSRND77Pdh0jypFsVBcwwNOFY5ZiNjk00Z288V82Ja+zU7JgI1rn5ATlk41II+PXUtdfhmmuuwebWGmZn5zAxUcX66jIaNfLF+rjx1rtECrx85ln0W3XNyfz+48gVyzh06JA0DL3xKGp89OGH1fF4Ye9BXL54Dq3NS1aDXZzGgaMnNY9rq8syZdnUAM1GU2dwZrLkBvoZpMOekk6N+rZiciat5KP815//ziSqIuwQUivoppo2NTeCeXczSqPOu+pY7b834ELagQkJP/vLSkkNmaOU8e+0pXSoKCjqMcJMenU/7nnft6Pf2UGjZWgWsd3hsCe8emdjw8kTLQmWtWvmrjWP02yxOZb8T4I+zzmhGTFP2QiJKrLzDglBPxpRguh3iOPmJ+QxqZKy9GppghqqjLfde69ds83zQbMoVytaTFasVqozow5Q3HV0Lq+/5Q70Wh1x6evbV6U5D5+4VZNPPjmdVDsdyMptv/DQQ5jU4Xd7sbWxgtrVc6i1apicP6bUMcda49mpTXaeaongQLw+V54VtVspzWSI7Y2r5tekmYqeMELGf/9F9kET3OMkPe/d4VxsoWVaLMNwhdCovYNpOU2hkhCEuaPO2tpRmJPDybfLqwGxeox6aa4awQzVpyWXTuPU130LtjpsoleX3SNEyd5xW5tb2FhdQTLoOH5uxEIuaqdDLNwiAnnebPQeDVr7xLG9/4rCoYHIlJEGDWhW2pr0q4nyqE6d5ufmm2/GwX3k0PdF0ZXjxRMH+fBeU85Qi1jC6soVHSBPUn5UuzS3N3HkhtO4dPY8Bt06NtcuCTy68dZ7sF3bxpEjR3RSImFTWhCO60uf/zymZuYwNbuIrY1VbC29it6wh5m9J7Bn7wHVfK1dPS+NOzs3g1aTMHMH+cqsauTps2ysr6K5sy56mBrv8Yhp+kh/8ts/4H3QbCFUye8Hh9mC+lGAYyfDKhRLeeMcnbgzVP438F1CjwJivGVlnE1l8pSo97ZMgxPuGPqo9CYzgeqJN2qhGVq0CBgM+qpDI6mOtCjmzDfW1zA7M6NDaKKihF2XVP/k7TEMJCGyV1S8ywklXYgPTRvLF0/lLZQKKGSyuPGGG/Du9/4LhXWdTl0EfkPlGBV0lQ3kiwwcqnU+Kz1fmbp0GitLlzC7Z49OGZC6L2Rx9cJFXHPtdVheXkKqR422g6Tfwb6jp2RCWFBRLtuYTY0n+MKDn8P0zCIq07No19ewdO6ryoQdPH6bPPJOc0sHwHaHwPTstNLK/V4TufIMZmfmNa619avi3ak8macPq8Chi9SHf+dHRottIZf3J1HHwziT2k5mGLEhBe0ZnCreGp0kPyhUjEo/RMXAA5oDU+8Ww6Z1noaYrN7OcgSqDFNo5efQyS+g2W6g120pxqYd7zQaaDV3pKZ6ZL2y1kq4vbVfZm7aTtyzXR4ghQANP6ScEOTMzDTWV1clnG99y73Yu3efaYheG7fd9WbVk3OxL1+8LEHrdpog/6xcrSppEW1G5Cc455sTWd/awMziohaRqrY6VcXls2ex//BhrKxela/BoorlC6+iunAIczPzYHRSqfD4KFPj1C5c7AOHjomHT01QX19Gq0Ou+M2YmZ7FkjgCqyhVyRGfx/bGhnh9E9N7MDU5q8UmgsYTkzkHC3v3iU7FRj+pD3/oRxPtwniZiR21QTYQwc/zEp4ah5fa7uBLB6V6laPgVe+sFDndKGS3YwYtAxSokmBFaQ1ChoYuDZmTTU1iY7OJrfqmKE47m+tsrYB2py6An+8jt9zgyzTyaibIrhAFUW/Z8oKeN5242s46zp05o5OD5YB5XzPrMgS0egNcunwF/+67vwf33PMmdfl/5pmnMTc9qaggSn051kbdNAjPqpYvkIJUJ/GAyWpVOALHUSpTnW5gbnYaV5eXsdNo4Prrr7fvazu4/ba7jSY9wR7ljAKsCPHBBx/EqVM3YG1tXdy+2uaqophD192qg1fPnXkG2QSY2seESB61zW3UN1cxtecgZqbnVQ1y9fIl60RZLBnbKE50+JPf/qEkCgREY/VWjdEPk7syXsJ5/Sxt6/tlQqKe2+y0pNaNFAw/US96aXpvci66drtfUI4Z0SQ/F5rHJUl4vM3ygWtuxeKho3j2madw4eISVq5exZXlS3Lc1Bd1dhYnr70OxWwa1UpJMXJc3zh4ea8qoZcgN13OA3ciNYQa1w/TaPUH+PgnPoFbbrkD//7934/6zjr+/u8/gce+8iVzbPw4BjmTxKjzBfHv6E2fOHlCLBoVEKiYzzooMKTiTQnt8kU0jZWdWyR4qClRWTa7Up2wolB30D73uc/h5MnrsHR5SVU4w14T/e4A+07cjG69jo218/IbZvYfFBeP8DFbWk/M7cXePQews7OB2tam5fRlwzkHnpn72z/8aanxAOwjTKKaVk9MERVYrWidjvRSQsEWNGykcrFjjdnMsTPnbVxpWBtn7zzgxxf1ujxxqCTkSCfg+HX3n7wVB/YfRKu2jVy5irnFPejq8BlDuRhFMDR76cmnlOyQifAyXFtb4/AG6udDdxKenxDkDNLBMAfCive9412oba7ghWeexSuvvjRKDgk1pBZKLEMXzeLJsKEfEXRg3mNyakr2mKElNYyYs/W6wkzGv9RGrVYPr3vDG9SEiLmJhKnWYYJHHn3UBHYwRLtZUyODZquDI8euxfLlC+g2a3JoF/fvw8b6ppVZnz+Lyfm9mJmdx9raFW2GcnXaDnuX752oKDD18T/9Oc96xaLEQRu2IHTVY+G4+GKMyMZ46exoMQ0UiMW1isZd+dC1YrZdnYcNZ77ZeG86ZXOUATp43e2YmZlDu76NVg+45uRJk3T2YvF66VaziacfeUSTZbVc5L7HgY8mbAGt8jMqDBiZJdvsSln2SKIs4u4336MzPK5cvIiVlSVD8lhPXSAtyzo5jkwQixG8S6OlVXkd4tI0N9ZhgYJAweDPtPkkVcq5K07ge97/flxz5JhCKAI/HOcjX3kEO7UaSjyLs93E1GRF9fB0tLrNBiaKOVXDTs/PY3V1HYcPH8aV82dQnl4Qf2Dl6iWU8gVx0phfiDPAei0u9of/s+9sSyJwN5jjZd0LvARaDlks+rhaJy4rmk5sei/U293NVNbet2t0wIqfejvWEE622lmgUTZz9NQd4kqz9HRzcxu33nan6EN9LwgkiEsy4PNPPAHjjscZnS6oLm3xe9M+u2duywt2fjzbhPLnm+5+HTavXMH66gq2ttcFCAlhcx5ZtJuyyfImc+54RuPa2OWMAthjbhxyVeTC1hq9Pk6dvg33ft3XabcGBflXf/VXsb25hTvvuh0zs9PSIoRl2W2KHZwD++dYGT9rnaghU8DUzDQ2NjbF0WPju+iwVC6woH8LqU/+5S9rZ4fKDRUbReheyTc6fZ04ehh9U6XehMa98dHnojmNfm9N9ETrkZ0mxkwN63XVbvt1cLiK3kzLnLjpbhRLRXD38nD1O+96I5JhV8QH+ges/OA1n+VikxDo6dlx8zFuRsxRsVMLOOlW62VsWXK3KLQ33nU31i9dxubGGhrNbSUQQiEpDeu9xSJEDWaqJYeM/x5HJGqR3dkN4CoqRukLTc0v4r63fb2gz26jJkH8h099SpwAopTtVlPPvr29uUtXJmihA+ZSgqzvu+8+1Ld3UCiXlG2k+aht76hogI6q2Dre/Sn16b/6oGlXV8dsnRFVhoq7YWCFuFGOhu2abtsZHCQJDeEcGcgSoIqlEE2VxiEzpt9JXrTT4Omhs5uQdxvy9OO1N98tpIxNbzc2d3DrbXcDSR+dtpEWCMgQwHjpxedEpzWYNHaupSo5vjixwMa/Cxrp++iE3DcTdPr1r8fy+fOqH6cTx6DTHDM7mUDM20gWceGdzCAz5R0gomOSiIuuScRC8ffaGEijmcBb3v4eVXU0t9Z03ccefxy1Rt2Yq85eVX23OkuRjGnnoZHvTu4AfQGdlUrT0TUYuNu2UwtOnDgpp3Bxcd5qyD71l7+h0Mt2HA8xsSZpRKFMPXtxwKhPib1P6tDroQlUkJkSXXCDdWEPz2YzfmqdN3qLUMwOHkvbGWx8qQGvgTH8/ckb7/TzNbjYNdxy613I8HRf2h9fbGLNr778guwcXxEh0GdQBYvzxU2VjqnwMSxAdeCevrrlDW/A0pkzKmC0fqm77bkoKrTB6tbsr3EUTjZ9LFctyFjQoh3hZEJj41AkkCvjbe94L7r1DWytXpEwPPfC83aWp1pVG8AVTXEZbYRGMg1h1SnBqOUCc/HJ3AmyhX5uNc0p/cSf/1qiRQ1P2rsKEQZUJkdlMFbgZ573bvM3O/PKbqgDUehgSQ17LjgcNnfOwlFidkgagR2FoxhdYZA5TKQv8+up03eKSUpEbWNzE7fe8Tqp0XZzZ+R4MYw69+orst100kYayk/dNQKGTdiIheI2llpD75fmsTHfcMeduHzuDJo7NU0QkS2xXvzc6+C0x7OEBov7aq60820xdGBtHGrLa7Cu24PP3jCNe97xbgyaTWxcPa/fsuecAVCR0DGuqti23lvNSpssK2lA0mudYwaaIm26r0HsXJnLB//+vxso6lAmOwT7Jhsttv4uAiJ3+lj7Z1eJRtAzMMVjldFiCK/2npzhrTOjxsEqc+axLwWHfULMKzfu+nU33+HYb1uY8Onb7lSIxpZdro+lwi6cPydIlU6aqVNbHMX10VB+jEQYioQecoSOAfjceNedWDpzFvWdHfMxvADBivt3SUu249wshB13tW6pYkvnkshh2IVrQ/YRVTjIurIEb/7692ix15bPSdjOnLHjLWNnhjDp7G3vrhRahfehWuecGF/d2EVc7DA7ETnIdHzm47+XMDgfSv34PyfmaZF0UhzPf/RmMxa4CfHSronuAj6ZvImdOGelqqPJVAdfO+A1doEWX9CrxMkaqovsZ6f63va6N2Nnh2yMLlbX1rD/4GEcPHgE7caO4mpRfns9XL50CVubm+Kgx3LwOgQ4RlI/5liJTOiHoclPdDVObXP9LTdj+dJlMWnIXo0+M+HHBIEhTvIbuWxxGq6r6NGCeZM+Cz0t2WSwM88USeMt73gPeu021pfOCjc4f+6MLbZ7/+FjKKtHAfFW3LbBDGJVqYo2kB9O5+FmNCaK45hTn/rb31EMUSyzH7j5nYb5+jmY0TpSYZLtCd5InQ7Ey7JSHCMKGL2YixkQbOw07QS/VrAzQ3p1Yg6rJxw2NcnN4vSdr8fm5roQI+5sxuF33/1GtOm5wjQQr7G8dEU7W2fZOu891DMfSrsjcHkXKIVSLqD8W4BJR05cg621DaytXFFPEiFRHFsY9TFnVnVZrloDHYxdZ6cGBbRsjeN3Y347S6SHDO5953vEe1+7fEaLfe7Mq4rVJf5+T/lI1ppAOL11d6TZMc0YZA3RrLxvfKzVa6KRz/7D7wsuDXqNUYqNVmyOWCBj9tCjzkTqG8qdGylOs7k6scZzmrb7DR5VViv8Al8AMUIlheYV6+jBqCbVzn4TVtdW1FNlbXUV3d4Q97zlbei22KbROvJz0VZXVnHl8mVRbCOc0iLpQBpXoe4oUXeF+jaBsNEJ8k2l0Wy38cd/9Ee4++7bsY+JDR8bif969miU4/6KnWoQjFwzcdG3xZJAMbN+JFMQHYnLI4Ove8f7MOh2sXLpqxLKC+fOGiHSVf04UBU5i5G/4AUOfA+F3tg2u5z34BGYtkwj9bl//OPXhF6jvp8uwRZnGjFg1NGXUpqN8yzNSVMxgSNmYZ/ouQZyZuc8ewStE+fNhpla2z1wLVpPJEkGt73uDeKNE3VaW1tDu9XHvfe9HT0S6nqsDrHFXt/YwJWLl1R/TafFMl9GJjTeuFdwqurFgJAwLyNAiAxTb8BnThaBlK44dYahu332tG8cZ2k70M/T8uOVAjnUCX0yJxae2nvjUBrqoQze+Pb3Ydjt4erFl2VzL104PypTskNndzsvhUmKbBvVeFCYAwCIsNds9Wtp0akHPv3HCZvEcbEikRF2wj5odjeAjlGHP8XGpto5SOFkyrCYBiDqFUcbSfKVMTMzoZN6vM5bu+s1xQnWYJZlwjfedieuXFkSAZF9vtge+g1vfosQNMba8fCbW1u4dO78qLOhjd+gzXhZZskmWlThcC69gI4cPOLyjCgsRy0RN36dkn3m8UYyJeLqEOZY9N1FlTfgHrlpDyvCsMZ4pC7TQXvj13Nn97B66ava0ctXlrxvmrFr4npxX9G8YiMyeRKaw9GeCNMsNIOyfqbKE6Q+88n/mZi63T2OgWzQkPgIAeiI6Wxt503HJNruND0tD9CPNLJF9ERJADY6dshaPlscGWrcvGe1+VANOFROdN0Nt+DKlcsiGjJe5K3uuvtNKp9ts10jGZnDIXY2t7C0tKTF3t0NnJTdHSV17tWRHKfxvmynh1Dy93TqZA+9twq/l9fL8NLHGyf0CGuIvqD+jCYg9j9UXYAsdhSym0hWtaQzeP1b3y2zd/XCS3LKrl694nQwW2gzpbsHxIiE4EWAHOO42tZ9RjlFrzVztFBj/cw//BFnWotkDEmLcUOiaHPU6DVtao7F+uqsMmYDxxeetczRRYg2kLHsru0O6lOoNNMXcRC7YlI/gJ1O2613vh6XLp5XcbmOccxkcdfdb7Z+afXaCPAgAHLxwsXRafajSXK0xjQNPK7AAAAgAElEQVSvh0puasxb9zg7doUgVMMR5Pw4SCP8OfBvPytr5MCS+KB22t5wncczSSgClTQCR+z8kXBwsQG84b73Soiunrf4+tKli6MTl0zQrKCB9xcnnKiemxRGH6G2Y6FDsEJj8hoSCP578B8/nNhxjP7gzh6hNx8XEgDiKpHzF2dHMakfGoEDVmd890AD4YrEF+fT4j+2prSzSEjmkzepigqj5cSk5PMl3HT6Nly8eAbNWl0IGXfg9TfdgcpkVa24wtPk37mzFYo4C3bX8x1pcn0TDiHVdnw+nMj4uxweXyA70NVACk+YasxU9zIjDIc8XtdZ2wolY0fSNHT8aAr7tKAdJX2ETeL1971P110+94IW++LF82aHw79RGOzZRvWIsYPkLTHz2ub7Sj2PHEKzmnHagFDSz//TR/ycdPPiVJ3IAckxsA5CmhTufH719GE81CiTNLbIeix3vJi14e6WpvAMWZgIo0BZmYyFDLsxOG32DTedxoWLBDi27RhmAi8Ts7jpphuxvbkyMjU8Punc2bPujVvYGBy0sFcGUY6Lnjkv2oVj7SflTwgxtL9FoY5Br6aZI4YOkmOobd4rMoYyYd7VP7xyhXBuhzWSYYJjN9yJ+YUFLJ99XkJx6dIFT8zsEkkS1xaMDKKq1Ha9JX9Cc4+bFX3v8xtRTurBf/qI5mA8WcBBy5UXROdsEpEIqZbd4Pvp8qPdYS6It0o2BIfgCr/GGV0kPASiEzF2TJCpmzghwHb88eMnFFY98MBnMD8zrf7m7V4a3/QvvxU7G1clkRScdqOJJ554VIsklE/OmSNebqujowHllTnvXZ/EBCBsXxAwKBzWsM6OUQqKFT+vfi2+ix3NlyCrSCKQNkcIzY8wGrOcRO+faioshfmD1+DosWuwfJYdKmpYY6gpLWKJFUszO1FEWDjPzbYiC/V1k7Aa0STmdmS7vcFQYA2pLz34vxJzauyhTUpt0qRu2GBdyQlzZlQ3xPeN8dQIpqhk1h0fE9rd3t4SHnVGcI/WVVnYwlDdcX/aTd6/1ezgwsWLytpkSK0Z9lBvDfHP3vcvtLPpuHCR2IjvySfI8DAVqSOYvSWnhMpNk7xgn6jY/fKmvdWlhWzWuzvUfbBrHdUd/T52EcMqdV3gSSd8U2g+PxMkujSquTZbcuq4rOixDmTKU7iLIea5M1psljqNvH47RNPGz8+Lym3FDPaKGF5++2ixw2FmOXAwSCTsX37of8lmW7Yodl4U5zP+cFBE9un/a+vanuuurvM+siXLsrk4zTMdGAghJc0Y22BjoLSZ5rl56kuf+tfkodP/oy+ZydBppkmAkkkoNrbBKdB2aOMB27JsS7Isy/iiy+l8t73XUdEM2JaOfpe9117Xb31LXYzxtLvTwR4pSR9LgEZeVpvIk5QJtIYnSxJVoAiPCgRAGTpVePBnQizc79H2pJ1+/e32zb11xtpsf3n8qF358ss+WSdIVpLteGFyvWrBs9Gx1QzLEJWYoCejJ1QnF0gDa19LpQHqjKhFJoxQa288TyHYI0pGTcI0abtzi+3Ea6+3m1f+pz14uNlu375pG68hOVhPcdqonJo1wXvt0kGTyQ1zlMRifHEtAgP/+MN3kgrhZuGHkB580V4nVu2D1nSxWD8qy8zI1O53tZh/opU2C0nPO2AFfxbJfKjG/Sc8JkA8prHvc+2Vk2dZDHn0OM342+3alSs97MgIKJ7ylAvLCU6uoJuqMgVQalnjmkZYpU2W5jGO3oyI1GY9RamedAnPKBgBlgQAYrQBrquDMNd2JofaqTNvtLWrVwiWYHrYqNVoGBZhzHmukM5OngfohMUh19f+qCAUT57ZynO/+wWRKnFociFCiJ3qRFYLtyAQwOq8k7LtG8fESlBX4QYt2u6nt5kSywXWwpBxCKrTIAeeOEnQjG1VgmeunX7zr1gQQC8TrgPM981ry4ImdfuVCYBKZgw5hC0WsIGLY3oLLbBKrqlmqZ/NiFW/p+RTAh5SWaP6ugaqmwpsu/7tqlfSpTxYmKh+qJ149S0WQkDTvbGx3hEv40gNkASzcp6AoEepYazVuvMe3XYnawc1HrTJCFdU4406pdfZbbRjYdNAUkpt63Pao0T4kvbMueIGFqpBXYstG2SmJicpFFZgrPAAMOq99FyvvfmXpKcAVQe5UnYet6t/RNVoh/9WGFeRMlrsLB7Xx+YJz8AowA9dVTun7iH37Rx6pgNFjQOmS7gV/BHWA3TiVD8Y3j7u1zeIc7vAMgVth3U92E6++jaZHzfvrfNkax9k4uJYZk1xVX6vqGrlPGBf5LDFXPR7JtV7/sN/0TmK+q07ZueAC+1eLv1dthsnAMNJ1K9tUJ5TlXJsaj6nPJ3Zi4C9Vi+YHERsR8hnnLB3rK/TFOfxe6Cu/s53ScRD4va97bb89dV27x7w5KMql7q2RiaBv7Q8g/8aAVdoOODFiU6kqFyT90LSJynwJPoeJUfOjeiD2uwxO2Wp0Y3yReDRo8x55s2ftDsr19rdzVX2d3HsYuaTs4xc0rV9/Sv2L1UwPKfEQLG6BtoEmzf5+KNfWhvY1ibD5FOZE231L3XI/8+Rfjqgh8R0OhlyukAGD3uM6TScqxVbvSdmhJKnV8HERQeGPSyJJvGhaBfCxbz1wlI7eeo1MiHTmWq7beXqdQLzMk1eWkm7O4odKXJhBomotjnAVKatV+jkUIVpSAyPFMbAjqzNkkJNbE2CeY+TyGQAMjoZuqy5W/DEVeAgwufAQjvz5l+3zdvLbXVtpd0Bu7OdUzw7ng8jq6kNSvGoh4LVfyrIWWpVb3YO8uTiuV8RSox4MN7zrPxLavIL6c5E7hoLMsKA2d9KzMffcy4XQkfaSrSpGqCYe8bOzXrII3VL5KYF6e79x+3tH/+EuC1K8nSPNB5Qgdg2fTYmQCpdXrQ96V6lEkVHHDloCWgBYMz43LGHnPGl9ClOTNS3snWKh5FnZ77dzh7Sy2Ql3tPAG8wCwbVFSARPQA4UNvPlk2fb1vptjuVYX7vFe0k51CaMsgeZQNBDMK19F+p9Cgx97TzhF8//2o19Q8fFfZcS1qnqm20Ok3SI7BcQCcDYJHrDO2itfaiGOzaGuz2ocJbgaSAAsy+pxj1+z2kSXH9j61F78y9+3DZuL8s32ttt6+vrbR1jLayZ9LzJHThvwFh40Fv2iCK8KHZ8sAEsBvnm2EBQhuTa+X719mkryc6gUcbpfcv6wCuI40n8gEGIWOOXT73RtlZvtdXby+3uxpr6203Bid8H71miADwLINQcBxFHLQ0Y2WQntKANuHbOo0w+Pvcr48a1oYq2ZSP6ifZb4nvzC0JW5gTq1CTcGDavxsg4DVBlcsaCWvUm2rusmiD935BUeLOS2O5Cte2duXbi1TNtA6dgD1TVjQD61bVbXaYZYbg2YQnqJ7UKKN5JVJcgBhCsadaxlKgpdBTIQYKZcq4SStKOEh/6AbbjIBzQ9TAZQAT5aYHSlaft+6+cbvfvrLW1G1fbPYApe11cCS4Wh+y0Yj16+jNxvN86BzJ/ZjGgzum/fPrJ+/TGe87XKiRqNb8QFYV226ouqtrdpz1mBCI2T+p1oCFHBDAECCafaUerUiRzmFjh3E7QcB1qr5w63TbXV0lnhc1GVeyOwxY9B3qzTBvhWLg/X46odsZwXyWElFoc5EGs1ZcCDXVdSrbOlxPznjCOZV4lQsgOYZydfADhzxi5USUJRPjD195o32zcabevf9XubK5zs3ELMkfVAbR+NojIE08cJeKOJU+/x7etP01BiAAvXvgNN5ujkKIyi0cH0Bq+hG5UjRpf8H2wAbFR+3PN/Ey3s2Mel2J6PVbCL17fTkw2qsezOiszNeLJ3lw7ceYNOmRomwEVFurda+urM2FXMnYUqHjLAe7vW5nkxvPtekq0L9Ze7DEDoTxoLsBtLt61aB8mobxW1G5GfDLxEu44ok1R25cX/4MfneD1bl77st0hnQgcOCFMD3pONvYmpLYH5kWwHy2SZ0a/WOJ/ijsPixIstNkXzv96mrSe0p0eG8GN1WXYQOAZzIEWIc/dL+i71RM/CgujlDjgsb6uM3bJPwe5mQpVct2Kaw2AJHFKa6+cPkuqRoyMPAjH78GDtrJyvTtMqqPbZsXw+zlzOpMAyp8Jl7KIPZal0+I0qHMC1BzklgFJkNPNwIQDaMdcuzppoImY2vSJls4ZAEccoOdefJk+wvWv/ov1akQ2nLyEWjbsL4afu0NEiS3BrWhanOaWMI5iiEJJ5eO7N/7Jxfd6R8jMD913NfqmZgvwcLoYI6ePiDnzCnbDyRWqcn96tGqB5Md1kmvHpU5zCHPTXMeOyvmF9uLLJ4hU2drc4MlGFm7l5o2OF0tdW0I3SADY2xVOb6NjcjK6SQkg0smLaAVqtzQxWoDU8eFChVU5N3TG+ZTDJg2pJoqOI2tz7cixYxza9tX//ne7ufw1JxbSbNmHSpIIDpmG2TSSDsATUIg6Uqj0j+LQGrZMDBCe8dNL70+hluSAqBdbR9Y+kRMgWNioA0gKOwVdyYEdQsNfWlajgns4ZUjTQFoWtegFzKbIRimRoahN4Q2+xEwoTTO/+FT7/kvfaxvra+yUQBsQ+LWHRrFtdMIoaVTxgkeQMJoYU4+GY1nbd6qmx6IKqKiig/B64z26AHf1OTQaPoj2KHGrylZn+Pt0Z9ouf/FF+5uf/rTduHalXfz9b9t3jj3J+QfJjDG9y5aoxmgGIEgWeTxsjvjBRDhss7b/Yx9BDt+0Tf5w+QPS1ygLlLgl+12a9N0JghoqnAJwimUze2xpG8GUnoefiUZaeCxtYkIi60Z6uqlj25O1vOm6Dv8ywdaFvftb2+21s2fb2q3raqnZ2WnLN67xwYW8CdiwJhZ1/yAyldQaoEQKMdWkCzelb6tv/AgKVE0y5EfCaEfSCy7BVP9XNXFxqOqTra7ebh988G/t5PGX2xLYEiDkOLEGIdAEGlARcGgQrorHkdUDH5oig9Tgtd6mOMPJ5oPkQlalLKCzJQeDxlE8iJ2NLRinI7ZbiyeV5nRy/xMbqhYVLXYqO/SwS3IAzxLkClUZF1D57uScITo725N2/NSr7fbNa4T34HpQ4xAOaJioZIQq1AxpKS7v5yBToQz5VTCkVJuTtJqyqCqQpA5dHUuxUth/KSldLHFKwqoejnC2JksYpcB32d0207JnDXAtlQxi+AZ1jfEW2zucQwZoFt6LnSPBCYDwxxXL6lDOL5joCKFXjZmT1sTi4SEB36WtsXTizxj8bEZ+P6FSTz06hNCNh6qUDRd0SDEkXtQUlS6Q8HeceZMwZdYXBEA/Ovn6W+3m8lVgSLlRt26taHE8CObbMoI5BTFVaEmqz68WWzk2KnP63YkBB4/aYqfPBOYMX0ySlNJjDVsxIE8lysIeGJw8b6TcNZJO0n6D37xGBLTNHALPxXArspklQDO2s0NOuHtb95iKZqOCexnhXzFE+8OnH/Bk9w2HNDlbJVumJvpsthIk+jyrRQnF0ozmPHPQL0mpjkoQZosM1TnrIOhfeDC8PPovgi6hSvToIjiNsIEnz7xF/jEAnHEfqPEsdGL5qPP4EdFYET5ojapOa7go10WFGt6fm6PWpkQuNDJOzECFIudO79ydKGSz8xcFLSFpcQiUANq24zjajqMxs+manKCnjXCR/RkEufb6EYKCkpSQMnKrqYjDeWXZbJbnAhEuD8JeLmdw6oZn07PxgiHLaWHzuGdcRp0GKEBuEoP60BbcwwID6HU9WbugJ9FZwhAE6plqEz+bbz9CL9gaxkI+pucKB024OYdp6QFmbV5NinjAePhpeNMzJKmihnvNDpFGUZSQaESCykDHTfrcLJxId7pogfU93Pewiz5xDHNAcmDI6eJ5nMPZt0BZ02WdsjXSXhJysTS5X85FFDhyqk62Ptpicuniu+JUsXwn5qZnTika5bO8XCQuajwbSu1g+yhbaT0SRKUXVQkUdW0yBjX0iPAbniAFD5wGCRI3jIYKRNdcIWgP+sGfnyAPORiI8LV8Q0R1GuCq6hKEjjPLYJON6aID4znaCZ34bwq7bDcWcjbRkky6kiEJtxiuWhBjfxlaudFR3Z9qicY6UXNgpMbhxe608eCkJ67jzmd5YeL8cfMOmDQXc1p69+hen9pbBQN/R6jKwfCXPv5N3qKoKpXWuHnGnOUEx7mQsyUvOw5RVB3SfLAb8sQ1mTYmS6xC4u5OD1QnZvP1gv4Erhz8pVWNcnQkVOP0QHvm+Re4qWBTwtfNWyukn6A3ySxWAAvyVtP7VHFawZlhpHIydTpxo5iT5E5MQ9VG4CvXe48qm0yiT5WRPemw7KwUtuOBQDEK4LFOAqn4OEVtx9xWf6mPniZ0GcIoAYxGpq2HULDEabWU2LFWpTicmV8KnZhata2m09BbXUZlDJ/FaKI0ApL7k4wOJTwxL3naUxcwjQf5ZJ9u3BEErBpBLCRIQiqGRm2+PfEn323PPvccqSTxhRInrscMAMD729tkG8LG0dPmu3gRDaiP/dVwtREbd3SttRP+LSEbBQ8+OzabuYKR/lVUEpNh6k5DruCvJFNY07Cxw0Go5ARjU+P9x//JhufgAcwoBy5Jd534oZm0T5MLH/0rq1483oVdIBs/c+xl2fqm8WYHNMwktQWcZHCNcpSEpYs5Yo5zkMqW4GhhUapDe5EqOQbtO5QJCyEhSsjWOXTDS2AMIRrjTp89S55OfA+c33BQOILJbI1KWcqRxL2hbSKgSiIp0zcSOXIKs8AAEEbFwjT1EK33sMthGrWV8W69JOq05nAexeeuTXOiaF9KF9eMNoWwc/18GPJs+TlOblXz6XaJj9A10acX3p0KYTEQFUmu0AmxPY8nrGFPQwTojZY4mZOBZtKecnIY6/qUZL7IiKPtnTvMgfCgiiU7rWIB1ZDVssp9ILcDWO9UW13RlN6Nu6tkEEJ2j+zDYPhzxSxISy2iMk4anrrN7s2kN9PrhQWiEBotk/KmzMFgYooDV52umLeo/ZiebDYrab16WMD9xdPucbK/V0NevAM2P/kJYO/w/ELhylzVCCsagDabF+bpHl2JSONFv4v1aFRRdDId4xkpCjyV0psD6Ie/0zFQykhT64o9g4MWPDeegW4ZhrK5vpzSphZ+FDUEPFTv2Cuvnmkr167y5e5uronczYkdqjE3K8ZZVNyMcBJOHGrSek+ke/GFgkpMC+7BU4TnOuAikWktYeOl9r35hjhp2BycOxs/x+3MetnJ1MFBfludKTBP7Et3eKf9MG0XES0DRcRN5vQDHM5RtIr2JC22U8JB4cSBnpz78JeKswtTLz3yvZEZktrTw0hy8AAOLQy3ibSl8Wx42cp88TTCMwTkx4uEFRmqBpkSXR+4NQmF79VhROJbSYQA7rXjp063G1e/5qJt3d8gYgVCxdKsNUV6oiPhym0btEBEKhZdqBipSxHQJ2rgOAr3VGX+p5Aoo3Ajpw68brovpBFrgPdmehmzxgszFKpcMS34LBNYKSfjul1/SqBSWuY77Gl2N67fSXNc3NFUxZiWcXhpsy9+/B6LnWH94xksqqOnMp33jqOGFB4+BqaeWdugGVgKbVBnvt+WOO9aJzfM/iwPTveYhMClU8+G972I4kSHEkNbiJlQEjq0x/bOtJ0+c7bdurHMzQH98vr6Gm12TwyRqQnZJRHEQjUne8dqUkh7Jgca5lknjGKumc6oHDe0KjOGR1vSA00TTn93PO+0HkOYMVtLGyikqPyA0e0Slatr6oTCvMmpVVwvhKlgVPiKiYRgwy/Suks4a7TUEy5WL9xoCEnd7NjQ/FCGXW4lZAWSGbUGT5eDUuz49MDeN8DpTBtwVEzKopmDOUhwR4GCqp+w370+sD2AgIAIEepx8+cW2osv/Vm7uyZ2QHCRX7++zDHInNG5s026aPGaisRWeX45atgcYsvIqCBHM0PQsanyDVwx8nShhGVDaOVgIfqginU+H825+uwBhoP4PLBkAQlkrSEQ2fCUhKN2c/BynWQy8X1om5rBjOfdVbYrez22Z+jFk63TkpvGkajA9rSuYlIffh7JlIqEIKiYEs8RN+8xcWcDVp4Ym4CXxwMDyYm5GrhGkitwsLiAbmLTiXHNuKMolZR55pnnid7cxcjG7Yft9q1bYmBIWLgLFWlqjU5eo9HJQXsQLmQikRAJcBNcIOEkQA+HBSgCwgh4b4bajd5ybW6yWlgLCCiETHkJYMWlIdI8iaQLGvmjqnFtrgNO9UzBTodOZkbTCuTfKIGEZ4BpwM+zrvHQuwBks2OL8+ewJw6H7IFCF3Ni3WGoZn2JamR4h5HIJF6wcHHgEo7lMwT68T/E0wovSKVpcLwkVlkraJP8nDXi6bQdXnq6PX3saRK9ovEdDhoHssGjNEpDmkWxKE6HpuSJ7opwXla0RPADqUtrUJxJOnT22IMQSVO9FlKsSAk3Ewfn5NHj3xZB3UxBCNqyF5ZS6gUEWQPl2CJtxAvuo9hfMXRYDpPLx/tRU1mYoE0gBKHepM934fy7PY5KPJYTJifdRZJCCSkPO2KnP6v6CF1HBCcaItAibeDwvOvvihpT6UyoRhVCNB4i92WSBO2rjx+3g4eOtGf/9Fm2Au3ubLfVdbQEyfFDEoV14eku2RHiiCoxInADrquKuatXCBMJbHQPd6g4IVydiK5kt6zm5YXvtsXDmlVK/8CtuVgH2VRdm3l+1w5U+VPuQRnFsZZsP8JweAsl1gyjkbG+bFAwVGvUuZXNSddJNDQTM0hqZbOTcYlKr3ajH+GGmRaa5BrpRYkwdk1ORkhsArcdUJ44cvlcEgVJFQZUgJ9jQznv2qMaBpOCFTrGP8LxObjQXnjuhba6uiLmgqt/5IJT4OLFp5l9H/BwRssYANE99vCrOvkD3nD9TJtBzWGzpbDQwm+kT0LKqNfkGhA2xbGSI6vWXmUItykETASlrm6wJwWyx+HGFITN2Y2QMHS91h60ivMkPGBffPbvU0gWbqzyn9R0Xjqbig2A5xwg/0gc2GlzrjdqpSaEEuPGS8y196dgByugVGPgSLGjSSRQLbtmjVLn8eMnCDaEqn3n5//UfvjS8/LaCb5YEG2XB7+HmUGU13a+vE9Y8NFtOcq+FE6nP4n/DkOzt5hajuXLAtLs3RwqCPW0rFOyma3dq2k6QqpVu7ukE81mMJo1BIkPWKNSviH7ldw6NWlICwsMmg5aJDXNbPhw3H1me6aN9ihtMREAOQAmijfAQGHUKEAkNSoEptCQ+BPCFQdCp1d4ctko3XMmGgj0Ju01ZleEnf/nd95pZ86cbv/4Dz9rf/93f9sWD8+3xUOLnB8GbxueNuNSsCog/jVlCEMbb3TQKR0IWPq7uA1u8Y0GDL02n7Hi0p0jTZMFO1fpvLoNyZzobAVWQbiXJ5N3p6oHHYjbh2nWDJcCQzPeGeu4uLRkLZsSrBy43vi/73RPLl14b1pZimJ/ZZMVf2MjOLBlH8mNPlP6hVPJ8bG+u3G3PfX0U7LplHrFhUlyKMQTLzgkP6paDs8YDRmTEuHA1VSSVC/1Y87sRBPhw3ZwihLnNz7JiIkftKUlTNgB7xlCL/V7YeKuSAKM9nSbrwo26ekOl5uydez88OmjlvJ7xjbG58m/eZ0219bW1zgkhtqFhRiphK6u4/OUHEc1p3aKmJRK0Yoh3aNHjCggvNG0iumFQuUhKpypk0sX3p9ubm4yoTCcrlrBksUeIL0JHSV41wn6ZcNjmwPzGaBD2ShVYSCRrF512g6hNdNWo8+FL3WEY0m8xF/garFeiGQDxiIjiy3BTCZqfjIhXgsoEKxv4lRQXfPkmesFz/fNN1vMpYcbpfssLKjITmcqQA6CwBpKM6eDJQjcVEa6s1vmqGSjKRRutpDGEeZOTJFpNRoeU54pthtTgZL8GTBuJ19szyM0vBc2OxL57U6ZbiZ77hFNpeEbkqVwJCeieucSfgLj+u8rohWFpuJu5ZI9ycBCoSyXwQ8u0EcYR5Sga89hlBHnj+gLagxOk3LvimnxBRN3//5WO3xoUaB7xPHz8+3QPOLgbaVQd7XoOAAYldSnHIw17/6M1kOFHsKDwEQcjHotItG+ptgj4j/AhHDqMMeD/kkn1TPmb6YWoG5PxuNYN8dPoAUPlmCsDZ5JPDShCoFJo4N2+ZPf9s3GpmdTojKrg5bNrp57PNrYOth2Zc6GdqAtBidocN8Zv5S5GS44xGEj1bJDF9zTfaSdB1Q+geJ7OVomk7U9xKhGxZdqm03SvWYI8bzppWIee6IRj/MW3m67HSaBxTDpzhyO8RwqicYBlUPmvHRYD0ImaEh2h3V11gph/ygwKI6Y3A4nPp8VocCgueRmylPrzA7adIV9cFjjNPJk/8fl302JPCzzr5SEGHTGRajlWboPORs9q/5lnxlzLqonKaceJy1pPZ40Oyg1BOLfozatQUgQU8hsc7+Mn8pmRwPd37rfjhw9qkEpHuGgbNkA62Xj6Yi6GY+x+67CIWwe1b5LuECSJgYGGPLOnY127Nix/2f6IgjQz2n4i9qWdhnVO4aedvwQdiE7FzPFOFzODu8xYGI2qRMBMzmG8cA8w9T8Lip5iXhkFg4wvp98eumDGXxCbHNOeAXwRwhy2hmse2J8atjZCHnYvU6mGZmeZ8Eih73zOEP99+yJ8h7FAcLCQ+UlYpAfIMHqwuZ5liNe1/35Lv4c1X3meblJT8+g08HMFNbYyBPlx3MPwZ8hCIFSJSunRFBoJvX5/VqxC2k89jIlKbZ1HAZBmxSDay112jXgHZ+7t7nJwg5VPFuD9sQV68YFnHx8v5c6ocbjIWsBRzEdL5qXIpDPbSfDSYqNnG2pqfYDf8c1qhbQQBi03oxMnDzYQTyjQHH4CBRyjDGiFtImI5SS1BvAaK4xLBJ6v2BSxvuMal7i+TwTFjNdILDdMDlhJkz7boQ6WMpJKI8AAAdhSURBVHeFTPM9/Rqn7SGm2TLZokWOZ87nJ3wJFTxtWl2TCMY4SHD8nO9wf7g6QhVbU70/gokKBbj8VZk1NxaWfAk1xOXLv5/SPhtaEw6x2G+l8gZTQiQvdrtWYvAgyYpF3UeAcpry0hEYwXoH9kzJj9mxilGfta0X8SbOrainFL5xRkhaVL0IQbf0Re8/l6DqkMlOjAVPn5g1aY+5NQmIGss4M5qJEPO5g0MaT8UTrB9ULNYFEUzleckzVXufE571iTnVeqpfLHYYzI442VwXLazv6VYuv2tMwOSzzz7iZsvDEyYq3mtuPLJiY6pMNjvqvnrrWqJxklIQiGpXCJbWnrGxuSayXimPytFTokYxcwowOfXwgBH/Aq9u4rze751JQGFuHAmfoDxiampdOUmdYQORFxdiFT8TJaZBfGFWNudKjbBy7RD+5tBwhBRNgRJSWQtBqPT90cwY7nIsqPP5ps0A4RBKuHpOTQfsozhKQ2OHlGGz8eHqqWbzUz8epzykqFC5QY1kY7Upo+gxWoaG/R/9xFGvtQ5bncR45ji5meKjk5ci/igYxPGSWgRXqVOdTswM4cvfIoiBGAffpsORcIr3Mxl+/02364hFQdGLBFuqM4DGrBlMFd5V5rACE3WvmkmMd5/3UM1cdfZ68GifbVblAMuRC0NEogL+jgs+9Ds+//xc51SpH0p5MKiObE6kKDndqp5rPbyq8bHE+lskOLadoUahg8qmj2sPxCfGIIhZUClQePxaCBPjwvbbYQmNNq6TGrJSkE7d+lQmWRLnbzhW0tUiBxi5+pz4qn6x2XHWlMMPBNgJmd4TDm4ZIV5qwTo2/969LQpGZ2xy/h73TBkzZgIags7XnCpd1T/oG02NZ8QrNjtSk1NWN50pOvdJMzXKAWUhtk0hAY1pGBAumqmqKbJww2kbZdMqEJHq2PiYAZkQJVeGV6xTgRQu0SX2/BGC4GVUsx5hTH+GjGvEe6BZgfPHFCb2cMvJnzwP/qQ69vgFePO5djZoqOtBWJDTCUEJiie16W9zziJAua+c2j2GeEAE6T2Vas7BgBMatNDsgTKYz45sYvfJF1+cFw9anddRSlYjoaHm+AhGbJaVeMc/V6ejhh9V6rT4aQ0a6jhCNpw6lDrdb+wifjYuzxsBVSZPSQdWoAwqYJxpZ4mkcalU5cSYKuvBw4fUEuRutIOVEI4LzchE+Paoea/GjI8Th2q/TzLUveJkkcQP9RxBzmZn8/P9CBQg1keOLLloFKbkUaHTvjjTZh5Xric88//8XDZbLrw+GDWkgsUgcmNhxMWOvExV9yqciAqK0GSX2YT+UP6bed2OIEHixm1GrhvHo8c1hkerNtZasKnhHTZDi2xwIBGv0DI6BQinDh9eGsCA7n8Hj65wCM+IpEo2O2iQnETew5oDahYLOBoAM21wIGarxqwaLhmxmouoMbjWAKp+ND5mPaJpIgSgBHvyyaOMtSHJ/YAZCxw7zh1WnA0vT433mT2ZBIqw0XoBVprc+hNtkOZb/Vt56H5Dj3msKoZ22JmsEepI3qr5iGceCR8/F2xoVqWbu6yGHkUooRJRi0fOLoBJBR8WPlflWBErPK54huQa8g7yA8yYmNGI1hJxxMhs6CRLTqScqoH/jg+E90h0UgWY4bCLRtV5zufzp1S6+VFNeAAPPbTfSSbxmZFBq55xJEc4LcGH5GVrI0EAQ8fEpzbSmbId1zDcV2bQtVfWwQL5d+gngCiJk7V/w7UnmQ44xk50zeLwUvH0MDNYhEMkiEOodJA0mouHl8hJokze6GGTf+DZIrPGr2cBq9kQkFBCzejezmWEPJue39H1k6cfEYUEwKEVhxBopHUEJEIg1a4GSp1wMSly0KyjBX7fh4BTfQEgdXMh9hICMJMujWRp4VVPjuufF+nqPjXYzgIgz5WntcTY+G74TmP0qTWcqWMt24akdk7GpkvCR9twTnwWJPY/mw2nJeqf82bNTMgcOMuhYBnU6GcszsEF0UzVzc6192ukaBeZORMRWJtFSCMEw2fQy+XfEhTXsn0N2nN7/DtZF/8shy+Ck/tqr9CSrGIINS8STNCsPjwo+vJQhEwAanxspLzrYMJif+Nc4PuCz6rmTKkMrpr5ZJUsuTlWCTOJd6vW1H5xX5QZM1YqKjtOVcITLeAgxgkvSxy54cmbiNbsDTwnlPgQ9nlSoPlX8axy2NCgGF6xkf2iBpvF8/YTHRUPXtCcQDx3nLrYeTbulRFMSHAwDGQXrUqwOKXEoO3stKWjRzsQQSHfWMH8HUxK7D1zFm/A39y9KenyaGlV3Kmlocbria6OQiS7OkuxPbKD8F71QJ1+0r9E25yGP6u8uvFU/24zDYlrdVjiE6g47+S+a+PDdAxgdU5U7CliWXB2Yqgc4LoLwHujros6d6V4dmGB7feO1SNssPOY5Y2vsXnjpPJeU+H3EhYpATL4YhB/R4j7oeImSVvBK4eNX1wQ5psACg+hjQboPlCiJm72nAbYl0oe7TS+7/73fRjI9n85OQ8T7wFtAwAAAABJRU5ErkJggg=="/>
+        <xdr:cNvPr id="1038" name="AutoShape 14" descr="data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAHsAAACkCAYAAAC3r1GFAAAgAElEQVR4Xmy9B5Sl2VUe+t0c6t7KVZ3TdPfM9ISePIqDRhqhZAn8DMu8hXnPmGXAawHCZDDmwUMYk0GABcY2wQSBSBaSQBKDNJpRGk3OQTOdu7q6ctXN8X/r+/bet+7o+fbqVene/z//Ofvs8O1v75P6ylfuTwaDATKZHDKZDIbDIdLpNHK5HJIkQSqVQqFQ0Fe++Du+n7/j116vh1KppM91u11kUmn0ul1ks1lUqlV0Ox19bjAcYjgcAAkwTPi9XYfXKxaLun7cm+/n/XuDvq7fbbfR6/X1Pl4jneZYEiCd1ec5Xv7ni9eIMfIavC7vw1fcg99zrNlMBvVaDYP+ABOVCjqdDiYnJ7G+vo7+cICpqSmUy2Vdj/95bSRpNJoN/Y3XHQx6+prLZFGv11CpVHQvpNN6P+eB9+X99Cz+lXPG8fErr93v9/X+mAP+rt1u6/7xe36en4n38JHHfx4MbL1qtZq+JgO7ZjabQbFYQurRRz+TJACyvtgcDC/A/5zAmKj4ykXW4g046fZ3CklMLNcAyVDvyWSymkDekO/JZCgIPc46uFx68H6fP6JSqaLZbCCTztjkcuFgg09RQAYDDJNE10mlbHIyubx+jjHwPrwff8eJiYnm2PL5/GjSY3K5yFxwjovCx89SkPj+drercU9MTIwm2+YgrbEUikXdo9Np6bq9Dt8/0PizuSz6w+FIiDlPMU6TBKDVauna/Bs/z+cZF8zYWHr+VErvp4A1Gg1sbW3pd5VK2TadhDBBqWRj5TU5tkzKNif/a30eeeSzCW9EqaBUhzRmMiaNsWt5gZAwDoSf4QXGX3wgTjDfpwE2GppkLn08kIQ+AbLSHKYN4sFarbYmm/fkq8MBZzJoN1vo8/tsVg+RzmYwMzOja8YYOAl8qPHdHRPJa8Ru5vslKJkMEkp9xrQDBW44sPFo0pEaCXOz0USn28G+ffuktXRPLnCvp89QSMoTpp14T16f8xC7lb/jz3x/aAj+HEKgsQ+GWshWp439+/ePtGyMnfcZ9Hsab284sE3A3ZskyOZMI+dzuxsxFlnP0uuaUHGxbQdkkMvGg6eQplhwx2ezI9XDwYeKp3qhpPPv8Qq1rxtQLfUHSHH3+04P6YWEwXYIP8Ndwr/x//b2ttTOxEQF2byZEk5Es9mUFOt+aVPNMRG8X71eH/0cE8txUfXHK8yGFjpJkKdK5GK128hkM0hzTLwfhaBQ1L34GalvQIuhuTIjos/SJHXaHZTKBY2fgspdSIEYN4tUrRT8MIn8Wwidmb8U2u0OUukU8oXCyByFidI4+n3kc3kMYLs1TClNCe/ZbpugmrkbjjZNMZ8zIX7mmYcT7hqqU74K+bzZwIxJTbw4UP6ev6OEUgVJsoecexOOUCGyYbk8qKz5no3NdQ2CExFmQjug29X1ymWqnwES3xm0vnpwV/cxCqp1jqPX7vBxkc3nJQSctGq1OhrruI2L3c3J54Rwgig81CBSdy5wOZoPJBgkplI5YVxYCdtwiKYvYJg3PsfOzo7uqUV0/6DdbWsecrmChIjCzvmlLdd8pmyhzBylpJK5cfjM3ADtTlv+QzzDxsbGSHiq5Qn9jf7EuGngfIdW4XxwLkJ1x9+kbb/ylQeSMp0E38X8pe1YU9vhjPHBeSHZJ19sk54JORJUg8WiSbfZNu6+oSai26V6tuuFitNuGZrTw50sByudNtua0KY1sb21je2dHZSKRRw6dAirG+taBNpH2ihKeKjDuG44llxYTmjsjBi33i/NQ7tb0PWnJie1O+kzFMsVrK+tI1/IY35+fuRvxFyMa69mo4Ecn6/T0Rj17IlNfKfTs53X72sjcY6pwQqFnNQ+BWVlZUXjp/ks5vJaAy4kf8c55e/54nzKbGbMNNCMhXaKv8VGDBPKcfLznA9qPdnsxx57KOGH292+VEkpbxKdSnEf8UY2aDpwox3mNjkmOLzyojsLcsiovodDPSQH1u31sLW5qZv2B2aLudgUECrJGKQW39XpoD+UWjOv1zx/Si2FiLuF+jSdzqDb77k3PpQnigGwuGcR9Tq95kk5W/Ja+wOZjjTv7d5uJksHic5kHu1WC8ikJQx93y0lqdTE7pGixkvrs7LJYcYonM0mVldXUCwUtfuSlO14037uZfNGqZTsLn0AzpG0B4Bex7QOhY8CxMXms/Kz1CKT1arMDl+r6+t6Xr4nbDMFM3yEiFBC8MOZTj355BcTqhpkslJFGdDB4ETa0vZ6HQ2aaom2iu/lhHJgfJBQY1IX3M30SD2Ei5Aq7DE93xAgqTEP7ai+5Xi5d08JplXs9xP5EXxY7cApk9R+zx2gQR/JMNEC8R5JYiGWpCexHVEsFTHw8IxmI5fNabHtfnwiap8ChoNEO3B9Y10LMj83p5+7rbZMVofOkdtwOUU+rjATw56ZQfkrFNi8LUy300V/0Nd9ad/Hwz9+Nmx4q1GX2s8Vzcni83CMVPGcf96v1WhKC4bDG+8L7ztsdcyjaVWLKjS2Z198IqFNkgT1uihkcpK8YWKhQKgLTjofIn7mLih76KAwhwvsNl5T6HFpSLWkjB6jS608U9nOtNSSpLvXe02IRBulsML/ZuaFXrTZPE6IHoKeJr33rsX0nFhei3aWO4LPxWeKUIy7k2q81W5pJ4a3TO3DBdGOTZuqDDVqiwp0JVR2fwvV0nouhYa01VzU4RCFcmm0q/nMNCvhryhUpUD7HAlTGPakbrm4IQAjjZBOj6KWcDLNL8iNsIoILWOueL/Qlvydnv2p5x4RqFIulc1uwzzbcqkgCTdny8IVOSeuiqhCQqJ4oXBcQm3JexwMMOngQ3jo3FUCWuiM0V9JpxRiUUVxYSOc4PWnJyfNi4Q5TXpQJCjkC/LaeX8+JD1pxrdcKKp4TmIsFEO8drulxZVJoK2mk0YB6nYNtODOd+eQO1iefio9MkXUAAp5ej20uh19nhM5HkoVsjkJlRwlmqGUCW84TvGZiGBoMrtde26Fn7Is5vxyTOHAUaD47KGyuXBzc3OvCWUjnAuVH+qb742/6XpPP/eogkw5LcMBCrk8mrU6si6hqbQF5IWCxb5STZykUsnCKk4Mna9koAGN7ARBAvfeIzzjoLk4dPT4PqpIDmK7XhvFvfzM7MwMWu32KKzLc6L7nDhDybiLqRppTkpFQ6K0A4e07ebwaVe4g8j7Npst/Z0mioJRqVb0lYLNC3KHc2KlGt1eT9BLdmSO9+ecMIwUltDrax6klRJaDQN6KMC8Hk0HJYoCxleYNOogaaFOR5+nNy6zZ2/D/PzsSKOG4JvDa6/xWJ6fD78gMA5uAqGh6YzubethplWLzZ2hsCABOq02qpWKSSehR/q83ClpAwG4GNyx3DGx66QmcqZqAjyhMNTq9dd486PY1uFBugU0B4VSUXZ0HC0at4+h8kIoQ7VucXfT4XEAQ0JZNGiXoZs8dtdMXCyzm4kBNPTUM1TBpgWIehEmrUwY3KmFpOYo5PUzr5dn3I+UaRIHXei48aXQldfu9qShKFjTMzOjiGZkN31M1BS8PwEbLUqhgEa9gYmKhad8hWoObcnn5FgVkfR6Ei5uHL4/5t6wCEMWBU7Rdxmak5h66tnHkoBAOVmUODpOmXQKDC3MVqX1gFT18pZztDe2k/h3gg0UgMCF+X6qND68QhXChfLOzRSYM2UOoL6nL0CwJLHYnrY2Yn/6CozZOdGESTWRdK40Jj68LZjtPBfIlMW2HCvtOHetoNax8E82t0sVaVJvCF0GRPEYslBI+FwMnbhr+ZwUBMW57plzgTkHfF5BpA558rliXqYqVY2NWobCymcNDcdn1Wd890tTMqZniOvQzfT0tASJG5DzEoJuzrAJGsdvttxQtRBwrolpV4tkUi+8/IwjaLsgCgdEEF0OBBfL1Qe9VvNg9QtHwMzrJfTJRaEKlQfoi0nEZ2NzwxElG8y41MbgLTGRlwoM3Jzf2QLaAyREy2lfAallhm2cVH7WJm4gf0A+RD6vhSKerJ3q3jd3KLUBF1DXSlnSRzsjbQ6p7bAKehJYe1ZeK9RqxNpyHtMGJnEX8sXvhTJms2hw0YQZ0GegYAwVj4dQclEnpyYtOeTTyvFwiiLMpRAqWnL7G5uEfku9sTNyOu3vKdn78MCZhyBIQ8xEavyZF59OtIiZFPIZokwNvbndaqBcKGEw6KPoWLW8c0mK2Sg+kOBFd3CUpZmYGDkFFBpqCmZcwqYp5u6YrZH5cODGMjp5CY2841xOmoVj4TWofQK14wSGdqA24WfDWYoIIkIcU30ptDud0b1kagbEx7N6BoEghCzTad2Ln+H9+BniCwZYDLBTq7lQM2IxRDGik1TWsk0Ubl6bfoZ2snvcMZ4AP8zh7KM6NWXJIvoXBT4/zUxfmkJ+1MCwBjqTvP7U9PTImTREzoQtwmD+bmS6uhQUcxilgV4++5KEiCBARmrUEBxmcxT0p2jPbUcRXOC2swU39IuCwt9x0gjtlcplhWHh2PDGdQL8zaYGPlGZ0OcD2aIzxJ/lpPCaA3P0qpOTI7+B15eEc9CDvsKi8GojpjR1Y1omJpYIFe0bNUCn05ZfEF5xqG6ZBU9cUBtQi0i1e+aI9k8qME3YNJGGKJWKSIa2kLy/wKVCVosRjlK/w4wefYMsCDYF3Mz3M2oggra1tY2Oe/Czs7MygxGXB6bPZxF27iqeP0sQ220JFneurunp1LDdYSIVy1PLyWY//1TCC+RyWYM23bGhyrTQimogh/Qw0c7iwwp6c4mykMrsnh6eNtRVeG1nR6B+2DA+CCVND5LQqelJYmWvlRk1eJYf53hGgMWQKnoXiTJNZHlzLmAAGgrhaNv1ecPCeT8JL737HLFuy3QxxuZX/p2LaGAPowWOlwtroVOnZ37G0L3xiCzCpvO5OW+0n51O10wLkbY0Q7WugKq+A1S6n4dk/IZhF6OOgKQjvOQut8RMSiqcY+dzxqbgnEYoK83nDhqvR/vOr1wzCgId5Ugppx596pEk0Cthub2+FpXOkGDPrCUMUkyMM1HiMabCINlXUyN0lCSBvnDcoRQMOkemWgwjpvetzJDwdMavGUkdFzqIArHLLRwkNErEzAAOLgr/zpBJpoC73L3rVqcjIeHc8p7joQntI69BoRHSlBhAxPHH/ahOI1mTTpl2IronGzow7TaO7UcsbOrUEibUVFqklAMy/S7o4kWem8/ATcB5irCJX/lZjpfzwu8j8rFM3FDzzh0aYaG0WJ+hZl/+CZ+DIhs+Q2g5aVHOMX2OrzzxsBabEs3kAzOblvUpyIYw7JG7z90c6kJwqKl0hWeesjTPkHivQYMCMnyyeE3loxXSEK60XTk+6GBtmP9HreK5Y4kZUKvtaLG1kxxk4b1MJXeVaJAQuoaIxRMY4lkrM0kWr3Lx5StwEvs9MK6mA0cVST/DQk8TLu2uMUcp1HVMrrJ2SSJvXlEKIxJh8gyxnGDhmTV+Vo6TmxXZW0LGLoiBuMnhYx6AGEOwcTx219iYMWQmMaITwsaDwUhg+RwCv3zTpB5+/MsiL5hX20POSQv5vDkuXGzFa2RtkHLjoRQnmw+hz7ojQlvHvSc141SkwMM5cE4Y6UWUQEocU5sUsJBCxdF8KAdPtOMUqlhYRc1gnrQtgMXLWak8MyW0nwNPF+6SLwK8oE2kAIQTQ01C28nPa/cS5iyUNEFcAD53eODhcYd9DHAj7DavG3FxhEImtDaO8C3CxDUaNWmY0A5M1hAj4M90TCm4XGgKJ0OucAYDIg0oVQAPYWeaNUfslDhyUItaMfyY1GNPP+pMFYt9mSDnhxrNuhaYzgWlqpwv6uE5iAjutbPH+Gjc7bSLyiyNATDSAo6XCzcfZc2C/ODok1N0LMzi5Nv1OB6OY2enprw3BaxQKJoal49AEoGBJYwciGLxPZxkqr+AGyNRMA7YRMxLdWjYQErXpSaIxYisGxcu8PtwgGKxKbTB6qGm0AJ4WBhUKQoRx8+IhQIsP4SIH59xLEbnNRk2hRMs6Nk1JXludHjDBNIp5Pt4T3EISH4grE2giBh8Pi9TKij3iWceSyg5TGVyMFnu7I57fz2qtJYgSdocTly+UEK5zLQl1bqF/nzI0A6GsBm5kDtcUF/CHWuYeAAInHCCFoa42a6MGNESFvQwzQwo/CAE6ULEh+N/20H8m/JAcro0CQRcGC83GqOxxU4Nr5XPKgH0JBCvx8WlL6A42Yl9kXjg89GX4c+2aJaIiMWmg8YF4hgopAzBNzc3R7loOYtyuIxXJ6zdSYYUNGooJm20OMp7M09uiKRsuzuIyk0QtMmksbOzbSEI4+uJsogYEcJFXB+OM7GD1Jce/aJsNrHtGj88HEjd5tMJup22EvrJYIB8sYRSqYzSxASq1UmUJ6Y8xKKDYyqf6pA340LRVlG1cuI6XebELbnP0IYTJKTO0Z7AfkfeKBGxXneESAkJC9za0TeaAJoMjr3bY5zqSBi/IoASU9nKjrmpUa7aKVAUXu7+yJ5xYiIk5ELyvzYA05m9rjhoy8vLyGWY5m3ImYpEBdOvBw7st3yBzBnnxeJ2vm9udlZ+TrNFUqUJI22tOZ4MpxjimQOby+cUVnEHVzwCoqqTQJaK0mB8z6WLF0zbFkpm5sjedSda8+Kw68hmf/mxLyX8ZaO+g067jmGvIyZIPmcTORx0iOojRQaGXPoicoUiKlML8gRJdqA0kiJEOHUwNFQqGCfaCV1yy7bk/Fy4cAGLiwvYs2ePecEOH9KeinjgryAdctdzh8euNrtkSX9OEAkKVOMUDl6P/zlew9oTQY8kSWSFtqVQKhSxtramu3CMAUhEJDCeOQo1zK9rq1c02advuwOf/Ohf49a73iCHs9M2XDoyf+F/MKdgmT9T54pcHCfgV+IOnLdxti43bbtlISIXmxrXHEFuImozmxyxiJIEa2uGIzBvwfmi3S+VLWFFTaJMpUgWBqumHvzS5xLyoNu1bQx6bXQb22g2ami36yCLI5fLmFpk4l057RQq1UkgW/IwKytUh7TeoiQsh3K5guGgj1azhYcffhhveet9MgecUE4+NYFiWIVK3EGkPNmDmUNkHjOFicTDRsPIhJxsqubAyvk3OljdbkdmCJ6WLOSpRSioxptmOElSgBZ0OJR65cQyAgmTwPtywng92UDPpIWD1WvXsLm5gTe+5W34o9/7EN7zDd+MhESO7Z0RHsAJDQHu9Q13N66bRR1yNDNmvgwhsx1Oc2eQr+EMNJvUKPSsFW45Pp9JG75BU8DfUROb+bHsXIZhpwSKiaqszKbRr90UfvTjf5Vk0n3UNtfQbzfQbTN+LYgmw1evb+nMtHO4h4yrBZ4QB88jTbJDvojiRAXF4gRKpYoGJL5VviDItdHpeVrTmBOBo9PmcMEIhHCSRdFxZC5if+4+Tg7NQLvbcWpSRfE3QyXa2Ga9qc9ZmJdCtcpkRV8U2vg9J4PcdArG1tamcHZOEjNh/EwQB8JciF3rW4mfbTS2UdvewA03344/+59/gG/51n+jzygJJC/egB7aawpKs1l/zZgsvcp8g6U9RcaUo2lzIoFwX4S7lbtaCaLQViOMwVk5bhKEySeGFWTyTEUXTJspbBsI8qVzq4TLX/zZf0u2tlfRqW9idqqCen1Hu6TXG2gnKF/NZEQkDpwJkmT5YMwDTyBfKiNXKCObLSCdLSKTy6BanRKVaXpyGps7dUPcFN7Q4zfHy0APc3I4mIhZd4n+fVQqEyIMcFE2tjZx9uxZLC0tKQ/Mscnm0oZlcyjm8zh27BiOHz+O6ekZdFpG/Y3EA2Nnzjb9kJ3ajpH0U4aARXjEcZjGsR3HCadz1GzsYGdzDdfdeCv++i/+DN/2r79LGiLoxeMevj1P1xiwYv0MtYvDJ1EWjQkPX/TAsoMsEk5faDja+OAO0P5qw4CgEfPvpEQXjXiS92oRYhTOy6P/QPuukPnDf/rBBANOWBubqysoTzhJYWjlJ5Q8euIcSHjc4chIEDI5qZpMtoBMlra7gHxxQna9Wp3GxOQCElJkCcP6i+GdqjGodpBCd2ATzAdReU82JwDlxZdewksvvYS1jTX9vecxcuzWcOzGVfHoHtz5JUYPBczPzOL06dO44/Y7BOoEZYcLFHbbgKTirsOWSrQjDB2DdnV9Yw2HT1yPhz57P97xvm82E0LOuUyMOUfhW9Cho8Mlm8xQivj5iPtmi8fn5e/DmVVenqZnQAEzDrrSlA6bCqyhqePadNoCkoQRgMCNcpNmNpywqSSVo2rSJb/xKz+eFLLMTfeRY/oysbonVmGYnbGgPC5CO0Q3n1IXjpI8cd0ASOdyUunZXBmV6iwW9h7FEAa+iKtFe0ywwGNvARwYKmy5cPkSnnnmGZw5c0YL0uoZm4NaRQ/ioVKABLHYoeqCIBDhEgkVfHCKFBedCRSmGMnEvOmmm6QFIg7ns0Y+X0BFwsXxWjKyaTZWsbp0Ea+756347D9+Cm++712iRtEfMNNjfLjIm9PTjjy9tJrnlhU1EATSHBAM4WLtEhW5Uw1MIQ/Acp00WSJe+m4NoCSfI9RMoqcnnpwzyKRPVI44XGj3+LX//P0JbVKxVECKnGXmdJkA8cUhmCV97xmeqMXiLjCuuZH7hCwxFOoPMTk5jUw6j/LUDKbnDmFyZlG5XQoMUbrI1jIuZCjz4osv4oXnn8dOoy5HLZIe8mYdirUFNI6a0Qu5YUzqRy/BmYwc7DchFBa3GzrHF8fBsIg7l/7I1NQ0bjx1CqdvuUVJlYjh47r83M72GlYvncPb3/3PcP+n78edb7pXBX6tesMWeWglReZMmXOpHcl/TvlSalh+gKlxIYb8zMDoTBEi8omocZjgiKcbkFYfxZBD80+4QfVMJC24phDsyhwFMQg3vYFmpn7xA9+TCIhPBihmWQJEN9/LdrSjzdBzNxIrV/VleIeUfDkkeaRdBXECaZyZCJia24NuUsSpW+6SNy4MmA816GNlZRVffvQrePXVV9Go1XVN2mYLxQzgtwW1laMW4WLzRS1iEmsPPVLd/n6S+cY/GzYw3isChvLmNE/GvEwPWVxYwVS1iltuuQWnTp0aZfc4ofXaOlYvnsPdb/46vPLyqzh2/U2y2TQtlrbkeI3kwBeflTl5YeacI3rVjoFHrK9lF2c9IyxD8XmAJq6OhRYWC2hRZauuwoTF5sTSzj4tUtkULoOxeyq62N3ZKaR+6QPflyhWywJDJh6YRRrS1hhFKQj7uyGRTbAyQp7jNpaG2fRR2pDFe4UK0vkqbr37rQIWRLYf9PHZBx/AU089iWa9MWJNWrxrFZ0Kl9xWxWLbw9kuEanPvW89rDMzYzEJqkilxxZ3Idjd2TZ2qVenKvNnyzkbIsg5IaBx04034fbbb8fO6hWsLl3AqZtvQa5YRaFcVdIj8TqrkTlIGS1bfgSdUa6E72gOWz7JWHgU8KuhjtSNxgW0/IFlBM2AkZJlSBsdM1HFXJOEuFui1lBN2/l0DFmk6MLxyz/3/oQDK5XzSDn91x6YWbCWFps7ke+PhAM/Ssg0dlxUUHCHh0dN9d5Psjh7cQXf9h3fJ/L9o08/g8cefwxXl68YgDJWSx1o2jh8GQscO9cEjjvbfIRQ7UNpZ+On0QSxIsScGtMMAlrGXiEUIUghWJaZM3iSU6a8fS6DifIEKqUK9i/M4NSNN+PW2+8UM1aOnlivu4wUwqaMDOhAEZMWS5Z2WaQI2wzyNZzRqw3j5BAurmWwGN6akFD70L5TG3EjjFBGpmhJn/Y5ZMREDSyOn7Sikys4D4Fs/uSP/9ukpKJwMk4oUgPk6FJ5WQztIyU0EhvipzG0cIaJr7iQLKnYtNVqK8eayeHVy1t45zf+n/jkpz+F8+cuaCe3O1TpVpyuHUYO1oi44EkT7TjPJXsFRnjd8uG1K6nGBhh4sZyx12yhtcjK8VqJsNlHI7jF38eFaFybjAtHwKb58gQI1jA+J4tmfmYex6+5BtccPmDeL3qkfouuJIFNzLHV7vTiwVjgKPYzgQzv2ahFgmY7lsAJuJNzTY89dr9COdaBZ4NGxXsa8ZGOXEC8xrBJI0XYlvyBX//Vn0zajQYmq+Sb9QxtoipKvG56wNJQBu4GBngkotooedJEZ+QtkqFhD6b0Jx2GXBk7/RKefv5ZrG1uIDUw4iCxbNpk2maFcz7rsYBhm2PhQtWG6chI4o0LpyyYCmK4iJT0XY41d7+WX3YuhVTGhGfcnsf3sdvHfYBIJ3Lxc1TtBZL3c0bu4KISfi2X5eFP5LK47fQNmJmwShBqiBFU6hUZdLgshbtrPhgDBz4fwEqMyWrJrALGVLz5TwRvbOGNI9DvGRaiOfDUcrBc+DMxc23WD/3mB5LN7XVMVSYsC6UkeQqH9h/Bvn17MDU1o52aLVWMJeElran00PK+nabiPe5WOhgE8pP+EINCFc+/chYvv/yyUpO0J60mHTDzsBV6yNu23Rn2OB6Uv1eO2RhyI0+aP4loPyq8J2Y8MJanY+KBfAnpc7LguJMW34f61jXdU9+140b0I0TJF/EDZIj/M+WbR67AxFBJDpbsvfyeDMrFKrKpIfbNVnDztddKEzDC6QtYoa9jzQqIVyszSIoVee6OM3Ac0nhjPooVRXhRorho1q4EKdvhUTYdqePYHBIW2vVg5Xz6H/4k6XaZ5aIt6WN1dVWkAuKvlCLaHbryzIpJUl18xIPOpOTFmlonamRgQJLL4eJmGy+9+KKcLg6e3mGzaYjPSK0ZlVrvsV1kYU+kN7ngI+ryWDWE/C7PiZvN4mJzZB5aOcGBJsfE3VKioSliYcMsjNvzEDZG/0aiMEdIi6SEQxHFUkVZQC4UVaS0U8YBGAqiV8jksmkUc1nMVSq45aaTgobTXpJLZyvoybLPo1IdY+2qqsRLltR1watCtEPdQeYGi9DLtoQ5hTJhgp4jXrcwL/UXf/RLSqdQCsx+GrbLeqSwlLcAACAASURBVGVKEFWFpQB366t5MzpYVD9cSEuRplApl5CvLqJXrOCVl7+K7Z1tT/dZxobCwCR/qGsuWDgY8RASHKFK9PAt8xYPZ7nrFLIeUlAABfprt7CyMoMBQ5mITp1HF5LOz47b43FPPDJc4dD1B8zpm2PFCSSOzs8TFqbJylcqUum5gvVqSWjC+kaUVIHgwHqqsFxI8zrsygGeLGXx7ne8HSxl5D1VvizqtFWrBpUrtJIxTswkBMxqxY6SeOcAmh/i0qy/8dmiPs1dFqR+4xd+ILHuOlbiQlBBXQdy5FSToGDeLKmzQqpUOG/0YpHbvc0EXaFBfhKl/dfiqYc/j3q7hW6LjpgJCz9HDjZBei6MFtE5zrHrAgkL7jYHH4BNCIF2WYQXopsx+LTnlKOUIZ7kxQgeesX1YyG/NpwLTRM73cIWCwNDy1CdcxMYPFxEkiNzp4wkYzufQsD38FqCdj3lmvI0roiVFM52C1tXL+H2G6/DO9/5Ts/W2diJZ/Mlb97JFRKUsZKrCKtIkmDVjsHYHoV4XxjLqRv3PIAcRQS/9cs/rG1n5D9ic27nvPoiiuRMzbgO99KfiANbrR0MhxnsP/12/N3f/SUyDnZQOxiNyJiTzDoZB4w/m80Sb83VdYRtob7DBsm++w4Zt62pUH9qCUVfg8O3/HHs4PAFIqQLJ2/cRxjH2GMMDKG0WxyNE1qo3LLVUTHTx8RPJl9Chg4se9Kwhj2VQb1hiR9OGGu4FF4hjXTSQ7NeR7u2iU5tE//ym78JJ48ftbptItxO+DAGi5mRICMGrs4oRxx4gkwwGFUl6iRDiMpkcxuVNJFdUzLlv37wP2ixVZfsZD05JE67FewmgMOACM5vgP02EH4uwczR2/DYc1/F6tIr9neVsUTLJ7NrDCcaDcKmJDdSEMx+M24OdR12VWqIVZNy4v7/VYzane5lWu2MIUtc7FDX4Wz972x0/C7s9bizpmuz84SXB+k6LlhRCWI8vDzSuRISpRfJiSvK8TThNAezXGE+voE+bWmvo2Cwtn4VrfqWHLef+g8/aowez9eP8geROxBl2KBYsW2UhevLUMlNUbxOyNXyF7wW7z1OqwoMI/WhX/mhJBZUgIX3BIv6qmBXWALe0pPuH5tXyf+dFvLH34L7P/a3SIYNDZxMC8F3TMnxMwJDDPK02m4Lk0wN79rmcFSsPHfXWePYYkxRQWnjME63TJbHcKGmww+I3bp7bbNv8dz83jJ4RpDQriSvzZEv+QxU105CMNvpoU62YOYuV0A6V0QhVxSIwQVniljz0++jTnIGG24NE2ytLmN7ZxXpwRA/+1M/6R0d6MgydUmVbpskiBARchl2bhiZxeduucliCQfWKckjs0aNOCTjN4/Ub/3iv08YQrCaIfhhu2GPYa8RAoUDZ5JvO55aodnroDZ5E557+CHUayvyUoOcR+FhJ0LtdudHEVMW0N8xcgFDMKk6955t4i15Eeo7FkEL57zvWLyAH9NZW0Q5bWMtu8a97XD2wqEZQZtj8Kny7EwFEqgcYdVWshTqn0V0NqHuw5C/njMiZrqQQy5rxREZr4ztscojGQgf315dRr2xjnwqg//4Yz/ila1dLSQXJgoNZJfFErW+K9FKLNp1EBs3pMyRNufnGZpsXj2/mgYGUh/8T9+nKk5WPoSBskm3zJDZM8szx1dzZAylYrhEqtLmxLV49itfRLOxpsExqWDCYzsyYL4g9wVRn5+ntgjnKHZbnoUEASOSOapWGUZb4kv23MEVLTpBBu4cx8/HwZH4Pr4K2Bgj/MeCh6NmKt18F4Ieso8Ou45/TuPwWD6XLig0Yx6/n5D4UGLnS5RLJEZah0JmyQrZNDZXCRevo5jJ4Sd++AcdLbPuipayNAdTIIwDMOGoKUHkfsS4mQptFlrMwBbWirtW5dxxsWUPnPX5tZ5qEP/dr3fyn4Hz2o3suNDpY/KGd+Lxzz+AixdeRNY9VO5wMk0M6SJD1CoUgjhnHja9cgM1DB40ocupoJBCZa42Q6qAT0cPOQb6K+4nNjDWqoPPFQscKjoctPHnDOctBM5UqAmVFbfbDhnVTHmZrqIRvx93eIoOWybHDJChXKRZFyc1hiafvdVGIZfG9toyavUNlHJ5/NSP/ahrNIIO1Epm7zkHyi94nbnh6bYfd5MlZsi4uagNhNx5HkB22pHMqC9P/ebPvz/hgKluwhGKna3p9fAodpOBdmzlZIxKJgJanT5Ofv2343P/9ABeefZRZNJUw6wVtvJdAhGhsg0T52TKuzDKMLsVhN11hEwqyEOvcDYi2c8HkkMXjXr4wKL5WLw5WgDPzH2tGh/f9eO7elfr2K6WgIAolJVARdGinM+BJzBYo6XSHysglLOWNgHJ5stC3bhjudDKQPXbqG2to1nbUi79R37g+1+jrYLepDVx51g5ctcsMUYrLdrtLxsmRqGqGEAUxF1QSprhN37ue9VAx+LBcFJMYsxT3m2foR3mHYXDzhK9ajVauO6d34Gnn3gWzz/xJXQ77NhgHuHkpBXDGxZuVRoR+1kmJ6V8dixQ5K3lhHmMKiKe57HNSfOiAW8UQGecjk/kt83W72a75FX/bwraQ+XLprmDE9/H5JFLxvdxh4emkJD3jDOnZxqShWPv0SKl89o8SOeQVTtN443xvflsVqyXTquOublZfO93faelI51PF4Idv4tx8e/jYwuTE8JhPpDVltNB5L2ClxDzl/qVD/w7lexavbEjVGNNVqN6kQ8RN+CFFhYWwBYQxWIeSSaHzuQJnLu8ise/8KAexpy6IeYXZ71wwOyWhVKmqqimVNM84lPvdn+IQgOOje0raYMCD4/sFheedj0ctkhphoqORY5F3Q0jvZPDGGWY4+JzRQgY6jBaXkdnhQA4ct5zRmgZm+8RIVSM7w1o046sSWPSnzVGSqrLxj/b4udff/11+OEf/EFfbGO2hJNq/lHAqJ5p9HZlaTmHDDONYxa1cdS6mltH56h9ogpUc/BLP/OdymczbolYkzsnVGXknMnbYq8RPvSo1ssTCCwZquX24NIO8MTnP4Mrly+OgILyBInwjEENFQpEzXZL3hrTpq2nWBD+xu1sOGJmUkIhW2Jf2ACT/DExY4iZdp+XvgYuEJM5vtPDHkc0EL5DaAIrKjRGy8jR89BHvVy8dZeySwlZKabOuU4K1cQxy6g0R/dXjqAuuPRd73o3/vk3vHdMjTMnb+2/FPJGaOpOqXnf5mkr7aww2Xh9Rllwe27fjHiC8WypX/zpf5swSJeKYTG351S5uATuc85bjpCF8bEe2u1jmlNNzzFVwvnuNB556LO48NWXkMomyInUDiwszo2AFAvx0t5vu6ydHdpDu9ix8NiNoY7DpBAXd1/JAIxUImGx1N5uY55Q5fE1JinEJa7Pn2PXCuN3vH40qeS5ec45FtxqoS29Glg2+WEquqcL7tGCqWAjTrCXaTTwEVU6ncKHPvQhlUiHmRPbhw7pWBp2V0CtBp73NQ3rFC0nMHCiJdzeL2a0+B45aSwf+In/OyFXiv27SbpXB6IRMS9tOLSyLN7wLpIQUYutBu9ZdIcJznXm8ORXHsa5l55Ft99GOrHWUlNTE1LZFDcurrzMPqE9a0jL3msGtJiHHwAHB8hdoqY3rE5UV0Dz3G3X7qpxg3stsRI7OhY6zAavN55wGXfUYnF31WhMqoFIRtm1/IBSvS41I+dJZLY0uh0nGoYdbvdUkkP1ru5L0XigVMQHP/hBoYCGVnr1ihMTuKjGOHGKkYeD+tmTM0ZiMAatSIteVGkIk7FUhcwpu5hC6o9/9/9J1HzVS2eEgdDekBJM58JPGMhmmOVJI3EUiQsshIv9vAg2II2vrnbxwvPP4qlHviSCvvBqVmeW2LzVPPKYVLOPhhoV8+wRYrxyld96OBOLEwLAWnH+jTtZsbtHBru7w9E9j+3Gw6zxRRy/7tdqgLh3CA0xcj4rd4xahgRI4YsgJ4222Om84deElookje1QFjQaF+/EyWvwH37sx91OBxXZulOpfwrDWmbt1FLL1HIIp1KqhRyGHWeiOOql4zjU9M+aBFohgiGRCls/9td/mBTLRWTUSwQCBZKEKTfr2zGi73oFQ3qw60QpNEmxwRtj3DSu1od48atn8ehDD2B1ZWmUiy6W8ihPGJPFvHEvuAtb64sbPkOYknEHSw/oD0xvM4SGYyTGzOvGZHxtDB3OllKKXgfN7yMBIgFyGz+uBew6VuhOSFRC5zy34I0x2aNIIW190MI+mgOaRTIIO2u5ezstIY1f//VfwczU9AhsspbfFs4JKQvbzHvGbg/AhbaakYznrpW/GrP1u2RM3ziujVMPff5+IX9q0KL2y757vGwm3H2Lei0nPY4hy6HxdFo/yeHxVy7jSw/8Iy6++qKpmEwa+VxWhQfRp4XccF5OdUjFDLpt6xca6pkTHs1aaU85iVTz47tw3KabJTPHJUKRWPiv1RKx2/lc4/cct7OKSZ0gEOxPYeXBb1NDH2eQuhYZjzLsnhmFWeY505QbCklG7Xd/93fjDW94nXPw9FcRMGge4h7RrYmXFzVpnA3rfPQe07DUKS64chIpcKo5G8rsGcnRk1kPP/JgQk/R0pykYxqYMALhnWLbb1uXWz6keeNx8k5KD8JS3VyuhOcuruIrX3wQLz39+AgUoNQyfjS8mXnznpAhkeDTAyR9CxnGqzPi4aJOy0AZE7RQw5EsYYO+r0XG4vOhHcIPCDX7tSp+3L6H4IzfS8wVz+Pzmv2ehakhMCEs0cFR3HkdTZHHgYMH8KZ77sGdd95h+RWRRUwTRe6BZkkOn0cQ0UslFt9Ewtil9PLDWbOMJVG0XWbqeMtt81E8qfT5z9+fsBMv7aHVPRmfigNSAl0XIqmcRXQseLOeXqxgZH5a2DbhTZ2pUcCVtW18+nOfw/NPPKLUpXUpsm75LMfhBLJVRKdjvcJZE8XidoUT8jDNQYtJCE95F3TZ7T8mQqEcOscH8plRV4TAv3fBEXOc+IpESahsmYgxtC3MQGiPuHcsfpiC2P1a9HYfe/fuxfu///2iHhsM5Pdy+rAEMG3PZxTh3TGxr7uIEuwU6Y3reV+WRRlgYk2AeS91qnAiYtC2rJWJbRoCQcIlIivorcVSD372kwmzVjqRJ2vdh1l7FQDEoGt4axSuST2pgsT7blLd+SEtjDFT6QKefOUM7v/E36Fe2xoxIwnAWO/SrOq2u11SZ62WizaXLzEyHXCJiYoJjh0+PtFy1EZJGh65YDZzHIXiIkZIFRBo7HK+N8xULGjYXA1ojIgYAjCeJ45dd8cdd+DffNu3e67AKjZpQ6PG21SpF+2JXGmYugmZVW8QhwgnkjtcvD0nDHLhtHO9k4L5GAyTdxeVi22JKzp0Rhahn0EBoGoX+vfpf/ibJM3QqdPWLstn85icncYLzz6FYcIwjJBnFXv37ZHtaNU3MUgySGVYrZlHZgDkK2wIYwxPqphXlrfw9x/9G6wuLwlDZ5E4ww+q6Xqt7g3r2BfNeoMOKInOlFEI70kRIy8ECXG3VktxtZzH6LliNnZ0ksAYOTGw5JjIWAC+N6jIdoSUYf29riF8/G9CbdpGCQ5f/NAEHCfr2n7mJ39KY2ZhgHqjD/qqTbfEhqVbWYynpvYD48rzFa1GuLBEIlUbzoZ9Y3kBnVDk7SrDbBCNMzqxaYg0mUHhs+ikBeMPcvz0j4zFk0Lqr/78D5Lq9Ax63bYkgdX611x7Eg/d/wkcP3EKi/sO4+WXX0Q+m8aBw0fx8tOP4/ipm3DxygomJyZw6dXnkJ+YQc/JJCwiT+XzuLzVwSMPfUYdE4kzVCtV84QdoCB0yvBASJDiCqtdGn+Zat/9XahNBXoKKSJDZHlmkiNjUUMtj9vmXe+eMazVnekeHpoY08N7sPjC8prjsWqo0sgw/b8/87OYqU6pw7HUvldi8Hk4FoavfFajEVGT2PtCg9gzMS9hVCRRmdzzj0NtKDChUaTxmPpVBMDuzz2rvuUpB+xVquY6lofv+r34GYFVH/nw/0hm5mbVe2t6egoXzp3DnXe/Dl/8p0+qo++RU7dgmcXvVy/h+tN34IXnnsDJ625Coz3EwsIcHn3gozhx+s0oqEVFHfv278fTX7of5cM34S8+/GEsXVpCPp9RO6geC/ac6cLJ4aFkQnpiQcc93rGFJl4VvTsNVCHQE0wWS4wYkGKCQVNjDppXcnqXYOamJQyBKbN6xc/90G7lzus6Bz1Sq9EiOrEMHR1F64OSYHJqGj/3sz+npEh446ERgnI1KgOWX8IerB3tYIJNpkms0Q0PYlPNupMuIoyjsLIxACneuXzBKkM8VCQMbfQuo25Rm/R40kGpKN+l06xbXThbpdCGs/PC3MI8dra3MT+/gLOvfhU3n74Vzz/5KNqNbVx7+xsx7PZx5sUnceTkDUpyFEtVzC4eQnlyAk9+7mOYmN2L/Ueu02IfO3YUjz7wcUzuO4LOsICP/t1HUaMq8dZV9DKFJMkeGUU2asis04QdTmbVIl5HNebIjHunEarJ3ku1pcSQMTVoFY2aPDXX3c1ta4d7VYWS+4RMM1YjxYlnSMjvdz16i5F5P3rXFk7mVaX5rne+Gwf37hsldsLBJFeNY1LbixZPTjCba9i4naQQfk803+NX7sDwJaiGubhsTBC+C7/yOjqZIA1t0si9B6N0e3vHyCNk/uq4Spbx9pD664/8fjIzO6u2FWxNwSTG8ZPX4crFC1i7/CoOXH8bFucW8NzjX0B5eg6TlUnUG01cc/I00rkMnvvypzTA46ffpAXau/8AXnziATRrNRw59UbMLsxic2MLTz76EL789BksXb6sXWGevrMynMkSB4lG191oWZl4q0h+jhQqPgiPfeAujxYUVu/sPcZGoIsd8Cq1SJUfdc1OiJQqde+fAIXh60Md+CoMWiR9o/bypTiYcbP4vEAubQ1riO2Hz3H06FHccMONygqye1TUG/EZFNuzOW+vp13ISwVMSgRRi+LnpfCrteMsqgcMhZj1d1w0CZu34OTOpkIzSDnB7MysasXYnSoO4su62Uj99V/+j4TF6LWdOqqTVaxeXcbhoyewvbmGK2efw+yBa3H0+LV48ckvoj8E9u87iq3aNvYdOI7iRBlfffJzaOxs4/ANd6HEHT87iwuvPouNy69i7vAp7D98rR7wxScfwKByAB/72Mdw+fKyqb2BdTgO+0Xpj7CEoQapwnzIyLZx8Ny1Ukm0/Q5YyJN2gbFsmLXVjOI4LZYxHV6T16ZajyTQbjLFD5rLG7NVbBSP7y0c9DCR2kQcNW8G7zn3cNCII3CcLHZg/7SJsp1lwrCM5nHYbSmKoa9jdKs0+sMu7Y4EgYe55Qs2N9T/1g/V6r7Y+ULOGokjjZqKKNVpiTVfbPbXrKPJDlM6Xbfgba0HSP35n/5uwqpEa59cBM+Xmp1flId86ZXnUJpawPEbbsH5l55Rw/mFPYfEpZqc2YuFxUWce/ExbK1cxsTiMezZd1iLvXzxPNYvP4t0YQLX3vI2dSB89bkvoNnq4vMvLeP5xx8fqR9BmNHPVOwV271c5JKfFMDfaZFzu0kaIWV+Qq86D3i2R4APTxQKh8lLYwngMOHCtKrRjiyhEWaBqcoAddQtSr3COXF2hgfbVZl9NB+DZT8sMOQiqZuTzibxhgEOdFBQeF/ZVPfCC/kSDh44iONH9mNl+SoOHTupnnArK1dRmShhdfmiHK3DR67BytUVnXaYKxZVhdlt1sVJLzAbmStg2GubZnNIt1CqamytTgvVShkNP6lPWolz9Vd/9jtJvkxyoDVutzjVmrGtXDwnZujJG2/F8tIFbK0sY2ZxrwSjOr2gU/GuXjqLnaUzQLGKhYPXYnZ2Adubq1h69REMBykcOf1mdUQ899LjaO9sYjs7j4985K9Q11FN5pUyZOFXWtp9+/Yr3hYzxI8nZlTGn6lo1ZMz2l97VaaFFlSnFk7xWlJvcaY2QaOx46oihqeaFN3XF5+2UPdxhzHUvFKq7jCypo0aYZzUEeDLOFizGzNb7xQV5jmGoNjeyZgEnt56772YmpyS8DY2LmNicg7XnLwJly+fxc76KvYcPIyt1VVkEx4ydxUz+49jbn4R68vn0ajtoFouQIfjFLhBymh3Gug0a+i1TdAIdnE+Un/xJ/8lId+Z+LUC+X5f9pDhQH19BcNUGvsOn1B/tPUrl5EpltUMNpUpYe/ePdhYX8ba2efFtZo7eB0W9hzAsN/Buee/qCMo9p28HYcOn8CVSy9j+/IZJOVF/PnH78eFM+fQ7Rnezfvu3bcfh09ci/m5eeRy1sEvuv30O9bnrMQDYZx2LBXrP3Px5HQZqXrk8Qu8oPCy+I5xrjea5zPy89FFOECX8URKNKoNgYmkCSnBStHGkY9RPDiWw+Z4IlY3xGs3JByhdrLhPF/T4F8ybCmQxw7OYX7vIdz9unuwvrKEKxfPYe+hw6htbKDb3NKc7T16E0rVKVw5/zLQazGzquKLfGUGM/OL2NlclZlg10rejzSpEos1//T3fzkR31nF3XYqnzrRF/LoNJuC6fbsPyJbsaZMFoeWRbZYxsL8HkFzK+eeV0gxufcYFvcfE3l96dXHsbO5ganFAzh6/BbU6ptYeuUZtb185lIT93/606jvbKDR6eOHfuKnUW8P0B9aX/B+t62meYwfCXiwebwWiIiR0CnGqhazdhjX09apM7E1j+VxVRFeqcpFaUMrciAwRE1g6VaDaMPTDR5XcMnioNnIkAmNU7WqMWIDsKHNpcPJ8NLOFfXTdrx8KFp18/ddnnnqfcfl7XtmXGeSqZdMTxSmQwcP4Z7X3Yna5oaAm15vRwvOse+95laZ3NrmEmqbV9H1as7yzF6kszwQponWzgpSgz62eYpvZRKTc3uQ+uPf+/kknS2gQM/RWQ18eC5Kp832WAkmpxcUpNNpo//KTZUrTmDf3gMCA66cfQHDfhPpyjwOHL4OxXwJaxdfwtrVcyhOT+PaU2/ULl8+/6zUYbtyBL/727+NlbU1fNcP/LjKaLa260ilzYwQwKF3WSa/LUlEqqCw8RpimGZJY2L/MaYQ+xh2efRCH722N9cbU8uWGrXr2kIbYNwmsqdG+EaJChiWX62Az1pYRIYvgI02QxgnSQaiJWqSw7KMcdXbTYV90aXJEiZ23rbF/vZ9HMhqHRSkPVRTwTH1UC0V8N6vvw95HajXQnNnW4zUvcdulTlbXzmP+tZVdFtNadvS9B6Z1+3NDaBXw9ryZWvik6RQnV1E6g9/62cSNpnLuo1MeUaF8KBaMOoQlylkeUh3r42GmCZZtdCYmJyRyqfdbuysI5cvYe/hU4JXV69exOblV8XeYAjGU9uvnHse9Z1VzB64Dn/2N5/EiVM3Y3pxn45n1IEvLEFVKGPg/wghEzrURSGbt3M1szxkhXGmgShpgjE89LxnXYLZs7TXZN6YkGRXNdGKad37p9dPDRKN9tSvLE+wYjCCcFlxysW26CCl7gahBfg7zoslM6xsmDvbnD5r6MfFEA7gvcKjC4Oa0PF0AF7DY2p+r2ILfc5r5HrWFLA6kcc3vOPt6LcaGPa7SJcncOyaWzBIp7B+5Ry2rlxgcY5M4fzB61EqTmCYdFDbWMba1SWFqRSwyvQCUn/wwf+YkKhAiaItYvsIhhNsXqf2Dil6x1UZeXYopoqU9BdLKFen5KVurS+hV6/JBMzuP475hUX1DVu/8JIWYM+J27G4cABXzjyPVnML5YlpPLvcRXlmDp2etd8S89QXkhk224l+aqA7TMzMyXazl6p77oasWSUoEyqceDaHS3kbCi4YPVnZzYT/DeumqdFB65HedWKAWlzJy/YjLbwgYChTMlCOOrSAOYK77BtpAbD7RFvevPkJ1pGY17TkhrUXCdqQBMd9iPBfDDJmVScPaAW+5Rvfi/SgZ+ZtagYHDl6PHoZYv3IejbUr6LGWPJNBdeGYmgT3ei1sXL2IAR01xuoTFZSn5pD6g1/70YROGNtIkFrERVZK06sp1JvDKx0M+7W0W5LKYnJ6CplcEd1WDTsbqzqFoDp/AAcOHlEP1NXzz7PfFqb2X4vZvfuxvXYVm8vn1PZyYt9NuLTdwOb6ttAuJUl27LhFmgp77Ta5s7DL6sO5s4lghSMU5bWMyyWILhQcL71QCpESFd6ey0piTCtQGFhTpSMn/WgK4eXMoHmKUhAoETcJgZU80RsPx5Dawzh1LHw0UkR49LxnOHcBgYawBFrGnyk00gxjPVzlHWWzeM+9b0C1lLPqmvwk9h44KlOyevkVNLau2rNkM6jOHQZDO4ZrO5uX0anXrCd8Lo+JyWmk/tsvfH/CKgZCRTlWIFKUrNLLzqygM5GyKkURERkzisGWQ5GdFgoTGPSaaNW20Go0QCeBi02MdvX8CwoBJhaO4NCx42g2a1i9+AobV6By4HpcqvWwvr5lZaaqELWJ4iIrJednafG+ERLxIQmSiEbknCum9Pi5qNfm7jOWqhMTiaDpyGg7tkH88yGUk9fnlIywMLA7sG4S2ZQVshMjUNJDXYzICvW0qHvhhoFbXpq7qOskD2kYp2AFeV+dFb6mTCcSKiGMwaAJX4Ff3/2W12P/4qzWZXrxKKbmFiVcq5dfRae2au23CnlMzh9BuWTtvzdWz4JUETmZ6Swq0zNIfeg/fXcigqHjyAmbzbK7AltLyzYzCc4qA3c2VFCQIJPn+ZhF2XpOXmN7045xqlaxsO+ornHlwsvoNtaQKc7iwPEbJCjrV86i3+mjtHgMm/2iuFRXr1wxRMhPD7BeXl0hZOEpR1ZMRx555YUQLSpELz5Uk9eoBGU9eJ4q11RmxOKWnuTCkCnCyfDzNpyDprM0WJbkvdA73ThegpSfFnLUbqQww05D4PUUQXS6fta3lSSHLQ8nLnZ34O2RJo0jKFyVuYDasVFxxOV77nsD9sxO6muDMwAAIABJREFUSkUX5w5g3+IBLeLm1bOobSxZGXRviPk9R1GZmsH21ibQ21I0pANwGx39PvVbP/sd1AFyoDgwNokXu8MdDJaeplM5JDnLVVN9m9NCmnAJ7A+mZCNVx9YWUrk8Fg8eEzy4fPEVNLeuIElP4NgN7kEunUW31UV25iBa2WnVSa0sL2uRGA9zt6lGKTPEsD806JBN5ssT4IlEskHecC8otOwWQc+a0Kd2ijxj8uDN+7bOidYWK5L+dK7YYpMTpaSHs2aiSWyUNxGv5vENwx6dKPY86arUNpoXtPtdMw/eKIj4dajigIEjPx8xdhAX6DyFoxhCbQ1sR2WaEuy3vek2LXapNIGpfddgbnpBuYzNlbMYtLcUmRQmJjE1sx/FiSo67SZWll5B3rVVNlfEgIWHH/rAdyZiOaQtO5RmGwmiUZ6xIQKsGmVWJqZTVmzOXaiOPEWUJspuuwaob22LZTo9u4Dq3CK21y6jvrksFHnx0CmUKhWsXTmPZn0HufIc2qX9SkRs7WwpyU71yyOQAokKtRyn+ubyhosTdaKNJVOTqUL5QGOlM2Ez6UOojIZwqx+uqkn1BjTMGFEzWJ8XClZeuLLial88xqqETOkEqTmfU5iUVnXnyrxpO4SdziCzXJEAEVbujFad3R1HZYjM4Od8e8M6TmQc16gx+CE0//xdb0KF53snKew7dBIL83sl1Mvnn0ONNps59HQWE7P7VRde21lDNunIBxLUW5kStzD1X372OxOzOVb0zZBLaFTBHDX2CleaMLFQQkcTqNk5Y/Gy7IF1sx+q9zYHWChXMLfvIHrNbaxcflU2ZfHIDZiZWcT2+pL6irAJfXfqGvkKXGweDcFqTsbtUaHoLbSlVjmZhFE5JmLcUc9katGQNf7nwgX9iMQJ29nBJPXKEYV5u6fvMU896HfkeCrP7nGwbDeb1PJ0wFJeKBfrzsLDVt83liA7kKJkhjtYTGTQOYquhMYPYzLeqFfRwcJy7pGPtwaC8iGcEcr+qd/yjW9DliatWMb8PvO4eZrP1sqrqG+tWPuNdA5z+46qgrTZ2EK7tqbjP3QC4YB14hWkfutnvt11hpXQBhtEh6MzvFExALnZWaTzVn8sJiSTD7Tn5K3xZKC8nYqrcy1KE5if36sdtXb5FbFVJvccxszcgjr4s3mMSIvlEwpVOmxDUa/LuYlcbuDVlvWx8ETd/dkf1Q84CcZKwkXgJDsi1uq27TQgr57kLlVhuoTaGTHe2sPOv+buMz67cs6eCrW4Oiv8nCRJOX19rzrReR5RgUJBs8pSMkeiEQl3KtOl7CYch89F01i69jI3znc3X4MttqzDAgWHWmeyMoH3vO1OTFan0RoMcejoKVQmJrFT28L60lfR7zYFnKTSZWlT9UEb9pB0G1hauiRNUixPYDhII/WbP/2vTY37ohqldRdW1NmWKo/M0OCpFFUYsnho1geMks42URaCMITIozI5h8rkJJbOP492s4nKwkHMzC5qR+6sLVviYvpa9NgxMWV8rJ4X64fHysmXSiY1iBAn04I6e9MSGNwd3Fl0jnhdlsFGaSwFNc77oAqLuF2qUud/GeOFcTX/RuFmbRuJAqq58lBqBIl6fM2TiMPmmrnY7aYcp/Ba41w3LXQO++yVZJTrqLSMggdreGMLLSrx6IjqtDTD1FQV/8c736S5nZxbxNTsfoVXPDu7sXEJnXZNglyd2oPK7KLYNIxqCKrwpGSmr3fqdZRLk9zZ36Fi/MjcREDPiVD44+CCtX5iC1s/c1pnhDA+ZjuJtJrCMUHP9BxDNoIwk/ML2GKXgc01ZAtF7D10UiqPP7MNZmX/ddjqG57MhHuj6Uc9DW0RR6GKdiorTzpIuEu7hpUTEVP7KLbS9J7oXLxI6PBZomCdpkjtuHg3jdvqrWk+goIbTQLkoHq7jvGwyey9dX7UGVrcJN4dOUgQ/MoIYLz/anjaUZAoCpXrU+5sgwGN2B9IG1uAc17vufs0juxbtM2RLePwsetFaNje2cTm1XPotWqoN9uYXdiPdHZCm6DXb2NjdUmhqDUw4Jrlkfq1n/y/VJ8ttTFWlmq4MGucrMsfU53y1kX5zWHo3QJ1oEqprF1ON39re0tYNosGipOzysisLZ1DtlDC/P6junnS62Fnex2Ti4exmSygM+Ahbzy1hhMPdFpNLabSrCsrQsbUUbHfwvbahtSikKiehU089ti47XZS4Hi1pdGS/MSByIJleaotbbkVHhi4stulwPhscYCLV0+6lpFH7WQ/2d047H3sFEE7etF4YSE0VmCw26dVrFvaZTpq6pC4W8BHLcCzWk7fcho3nziMTqsmBK5QncUij+FImGhpY3PlPHrNGjvJoDqziInKnO7RaO6g19rRQQHUVKRIsX9b6hd+9F8RNbbzPoTC++GnnguWeo/KSTVbpUfMHizehsIPbGOF8GR1Uk1pq1PTlldOpTAzN4+rF8+jN+xg76HrpHImiadfWcLk7CLWM3tF9WFMScePue0aKTU6M2tTCRFmgsjk5RENje0dqXvBlElw2g1vHq9uDApSLLx2ZZza5+UycVipOh6JyMIODFGf6ScI+yLuxskegqrbgrFbuctD3ZN9kuJCC//uW6/vsb7qTGqIaDFioBikGqzVfDaDt977Nhw5ehS5BNjavKjsI9X9/IETmJyeQ2o4lBrfuHpOY6YWzZd4tGNFgkuKdrOxiWG3Y4fJcjMih9Sbbj2U3H76JuxZnEW5wGMgbGcYsmTHOUnL+JlVVNuSfB4xIftt8CV42MpE2equqxXtNDam3X/oEFaXltDpt7D/AFG0JiqTU9hcX0OhmMdw6jp0kBOjIzhZdNSIVtG2Moxpt5totWroNNtqkcm/G1drt8JDp+xSCBMoHAv4MXaptFLWIFYdqRB9x7UQdppwf2AkiqhBD7ttTiNtOyfDW2RFoTyv56Wz0jKEPcWMTsk5ox7ghomW21UeLyV2ib2OHz2Kd73rnTrakX7H8089La0wOTcrz7+2eRk7W5tqaLD/6CkU6FUnJG3WsL58Fjwsjru2VJkBUkZy5GIPBy0Mve1GVwfDVZC65YYDyc52DZ1uH3vnp7BvYdKci2Qg7teeuTmxKKpVghpMORpRwFgtwqasFbPjuJwoeucKHZIheEYlJW91dQULe/ag3e6iPDktQiL9vurCYaxiHgl3sLJUHaUtZZO7jFlbaDUbqO1s6G+M5UmOCOyZE0Shi1NpFaOn2bynjEabJTNZxc/WoZ+JClOlPG6AgsoiCNavjRIgsJpoU+27rUWCjCDVOxiiFGd48z00H96TLCNUz2JrhWR+AnAqm0elmMVEtYiDC3tx/fU36Pip8ClUxpMCnnj0EQlloVpFv9XC1tplgGeDF4ooLxwWKbRR20aztYN2bUtzRH8qW6yiVK7aCcHtJrrtJhKCQATApE2ySH3vv7o3YTqvR8eDXYa9+ZyqCr0/mb7qRAErLdGBLf2hFnl6ahJ79u7RQSqGaLGSgtUQrGe2Qv04TqJa5Yl5fRQqVSFOxL6LE5PoVo+h1UuBNWeKibsdLQ4dL8boGxtrGrg87xbP/zLcOcJEqWOPkYm4EeUSEZD1awXrrM+QjQfAqgyHKFjBCIUsT2ZhgEgDNGEeOAU3OxbZ4E1r0MvPTfL0PyJnLhhWnsPr28HqFMZKtYo98wuyvRN54hCb6LR64gIUJmZxww03jLo+EKmjKfvyF76AieokSpOTWuy15fNqbstoZ/bQtfrabtaxvrGiEJbRMdkz1akF7XpD69qq8GFYxnFIjdP3+vkf+iZtEjZmV6rNCXW0wZwk4b7qprRbtald5z1MlaPyqg4V+fnpPTOzM7j2uuvEqCAIYIOwDj4E7SNVqQashTkkU0f1WcbqFBR+JQOD8XOzuY1+u6OfyaYUB9pP9RXgIgDD2leJBOAn7vCe6YxVTPa7BF94CkBJlaOBgKnvJ59HqVbadfNfmC3Ty7NbnFUlJzy2Vh8G92tYp8Wdye4Kx48dU/NZ1p2RYXLoyDVoNxs498LjSPptEGsvTC6iNDGtkwXjUHoWPfL5udiV6pTCrPWVZdRWz9uclWew9+Bx45HvbIrlQ4iaY2r3eiiXp1Am7yCblT3vd5mOrqtdds6Zralf+YlvVehFhUz4Ubli5oVVAdGjhTJnw20UmV4CKFxN8fd2Gp1liSIG5c6k/TLbbwT9bsfO/5pfXJQ22L9/vzx3kh6Ge06LVkumZiQSqKLIrWq0ttDheZs847vZsF2tQ8GNzMAXcXsKJl+BSRND77Pdh0jypFsVBcwwNOFY5ZiNjk00Z288V82Ja+zU7JgI1rn5ATlk41II+PXUtdfhmmuuwebWGmZn5zAxUcX66jIaNfLF+rjx1rtECrx85ln0W3XNyfz+48gVyzh06JA0DL3xKGp89OGH1fF4Ye9BXL54Dq3NS1aDXZzGgaMnNY9rq8syZdnUAM1GU2dwZrLkBvoZpMOekk6N+rZiciat5KP815//ziSqIuwQUivoppo2NTeCeXczSqPOu+pY7b834ELagQkJP/vLSkkNmaOU8e+0pXSoKCjqMcJMenU/7nnft6Pf2UGjZWgWsd3hsCe8emdjw8kTLQmWtWvmrjWP02yxOZb8T4I+zzmhGTFP2QiJKrLzDglBPxpRguh3iOPmJ+QxqZKy9GppghqqjLfde69ds83zQbMoVytaTFasVqozow5Q3HV0Lq+/5Q70Wh1x6evbV6U5D5+4VZNPPjmdVDsdyMptv/DQQ5jU4Xd7sbWxgtrVc6i1apicP6bUMcda49mpTXaeaongQLw+V54VtVspzWSI7Y2r5tekmYqeMELGf/9F9kET3OMkPe/d4VxsoWVaLMNwhdCovYNpOU2hkhCEuaPO2tpRmJPDybfLqwGxeox6aa4awQzVpyWXTuPU130LtjpsoleX3SNEyd5xW5tb2FhdQTLoOH5uxEIuaqdDLNwiAnnebPQeDVr7xLG9/4rCoYHIlJEGDWhW2pr0q4nyqE6d5ufmm2/GwX3k0PdF0ZXjxRMH+fBeU85Qi1jC6soVHSBPUn5UuzS3N3HkhtO4dPY8Bt06NtcuCTy68dZ7sF3bxpEjR3RSImFTWhCO60uf/zymZuYwNbuIrY1VbC29it6wh5m9J7Bn7wHVfK1dPS+NOzs3g1aTMHMH+cqsauTps2ysr6K5sy56mBrv8Yhp+kh/8ts/4H3QbCFUye8Hh9mC+lGAYyfDKhRLeeMcnbgzVP438F1CjwJivGVlnE1l8pSo97ZMgxPuGPqo9CYzgeqJN2qhGVq0CBgM+qpDI6mOtCjmzDfW1zA7M6NDaKKihF2XVP/k7TEMJCGyV1S8ywklXYgPTRvLF0/lLZQKKGSyuPGGG/Du9/4LhXWdTl0EfkPlGBV0lQ3kiwwcqnU+Kz1fmbp0GitLlzC7Z49OGZC6L2Rx9cJFXHPtdVheXkKqR422g6Tfwb6jp2RCWFBRLtuYTY0n+MKDn8P0zCIq07No19ewdO6ryoQdPH6bPPJOc0sHwHaHwPTstNLK/V4TufIMZmfmNa619avi3ak8macPq8Chi9SHf+dHRottIZf3J1HHwziT2k5mGLEhBe0ZnCreGp0kPyhUjEo/RMXAA5oDU+8Ww6Z1noaYrN7OcgSqDFNo5efQyS+g2W6g120pxqYd7zQaaDV3pKZ6ZL2y1kq4vbVfZm7aTtyzXR4ghQANP6ScEOTMzDTWV1clnG99y73Yu3efaYheG7fd9WbVk3OxL1+8LEHrdpog/6xcrSppEW1G5Cc455sTWd/awMziohaRqrY6VcXls2ex//BhrKxela/BoorlC6+iunAIczPzYHRSqfD4KFPj1C5c7AOHjomHT01QX19Gq0Ou+M2YmZ7FkjgCqyhVyRGfx/bGhnh9E9N7MDU5q8UmgsYTkzkHC3v3iU7FRj+pD3/oRxPtwniZiR21QTYQwc/zEp4ah5fa7uBLB6V6laPgVe+sFDndKGS3YwYtAxSokmBFaQ1ChoYuDZmTTU1iY7OJrfqmKE47m+tsrYB2py6An+8jt9zgyzTyaibIrhAFUW/Z8oKeN5242s46zp05o5OD5YB5XzPrMgS0egNcunwF/+67vwf33PMmdfl/5pmnMTc9qaggSn051kbdNAjPqpYvkIJUJ/GAyWpVOALHUSpTnW5gbnYaV5eXsdNo4Prrr7fvazu4/ba7jSY9wR7ljAKsCPHBBx/EqVM3YG1tXdy+2uaqophD192qg1fPnXkG2QSY2seESB61zW3UN1cxtecgZqbnVQ1y9fIl60RZLBnbKE50+JPf/qEkCgREY/VWjdEPk7syXsJ5/Sxt6/tlQqKe2+y0pNaNFAw/US96aXpvci66drtfUI4Z0SQ/F5rHJUl4vM3ygWtuxeKho3j2madw4eISVq5exZXlS3Lc1Bd1dhYnr70OxWwa1UpJMXJc3zh4ea8qoZcgN13OA3ciNYQa1w/TaPUH+PgnPoFbbrkD//7934/6zjr+/u8/gce+8iVzbPw4BjmTxKjzBfHv6E2fOHlCLBoVEKiYzzooMKTiTQnt8kU0jZWdWyR4qClRWTa7Up2wolB30D73uc/h5MnrsHR5SVU4w14T/e4A+07cjG69jo218/IbZvYfFBeP8DFbWk/M7cXePQews7OB2tam5fRlwzkHnpn72z/8aanxAOwjTKKaVk9MERVYrWidjvRSQsEWNGykcrFjjdnMsTPnbVxpWBtn7zzgxxf1ujxxqCTkSCfg+HX3n7wVB/YfRKu2jVy5irnFPejq8BlDuRhFMDR76cmnlOyQifAyXFtb4/AG6udDdxKenxDkDNLBMAfCive9412oba7ghWeexSuvvjRKDgk1pBZKLEMXzeLJsKEfEXRg3mNyakr2mKElNYyYs/W6wkzGv9RGrVYPr3vDG9SEiLmJhKnWYYJHHn3UBHYwRLtZUyODZquDI8euxfLlC+g2a3JoF/fvw8b6ppVZnz+Lyfm9mJmdx9raFW2GcnXaDnuX752oKDD18T/9Oc96xaLEQRu2IHTVY+G4+GKMyMZ46exoMQ0UiMW1isZd+dC1YrZdnYcNZ77ZeG86ZXOUATp43e2YmZlDu76NVg+45uRJk3T2YvF66VaziacfeUSTZbVc5L7HgY8mbAGt8jMqDBiZJdvsSln2SKIs4u4336MzPK5cvIiVlSVD8lhPXSAtyzo5jkwQixG8S6OlVXkd4tI0N9ZhgYJAweDPtPkkVcq5K07ge97/flxz5JhCKAI/HOcjX3kEO7UaSjyLs93E1GRF9fB0tLrNBiaKOVXDTs/PY3V1HYcPH8aV82dQnl4Qf2Dl6iWU8gVx0phfiDPAei0u9of/s+9sSyJwN5jjZd0LvARaDlks+rhaJy4rmk5sei/U293NVNbet2t0wIqfejvWEE622lmgUTZz9NQd4kqz9HRzcxu33nan6EN9LwgkiEsy4PNPPAHjjscZnS6oLm3xe9M+u2duywt2fjzbhPLnm+5+HTavXMH66gq2ttcFCAlhcx5ZtJuyyfImc+54RuPa2OWMAthjbhxyVeTC1hq9Pk6dvg33ft3XabcGBflXf/VXsb25hTvvuh0zs9PSIoRl2W2KHZwD++dYGT9rnaghU8DUzDQ2NjbF0WPju+iwVC6woH8LqU/+5S9rZ4fKDRUbReheyTc6fZ04ehh9U6XehMa98dHnojmNfm9N9ETrkZ0mxkwN63XVbvt1cLiK3kzLnLjpbhRLRXD38nD1O+96I5JhV8QH+ges/OA1n+VikxDo6dlx8zFuRsxRsVMLOOlW62VsWXK3KLQ33nU31i9dxubGGhrNbSUQQiEpDeu9xSJEDWaqJYeM/x5HJGqR3dkN4CoqRukLTc0v4r63fb2gz26jJkH8h099SpwAopTtVlPPvr29uUtXJmihA+ZSgqzvu+8+1Ld3UCiXlG2k+aht76hogI6q2Dre/Sn16b/6oGlXV8dsnRFVhoq7YWCFuFGOhu2abtsZHCQJDeEcGcgSoIqlEE2VxiEzpt9JXrTT4Omhs5uQdxvy9OO1N98tpIxNbzc2d3DrbXcDSR+dtpEWCMgQwHjpxedEpzWYNHaupSo5vjixwMa/Cxrp++iE3DcTdPr1r8fy+fOqH6cTx6DTHDM7mUDM20gWceGdzCAz5R0gomOSiIuuScRC8ffaGEijmcBb3v4eVXU0t9Z03ccefxy1Rt2Yq85eVX23OkuRjGnnoZHvTu4AfQGdlUrT0TUYuNu2UwtOnDgpp3Bxcd5qyD71l7+h0Mt2HA8xsSZpRKFMPXtxwKhPib1P6tDroQlUkJkSXXCDdWEPz2YzfmqdN3qLUMwOHkvbGWx8qQGvgTH8/ckb7/TzNbjYNdxy613I8HRf2h9fbGLNr778guwcXxEh0GdQBYvzxU2VjqnwMSxAdeCevrrlDW/A0pkzKmC0fqm77bkoKrTB6tbsr3EUTjZ9LFctyFjQoh3hZEJj41AkkCvjbe94L7r1DWytXpEwPPfC83aWp1pVG8AVTXEZbYRGMg1h1SnBqOUCc/HJ3AmyhX5uNc0p/cSf/1qiRQ1P2rsKEQZUJkdlMFbgZ573bvM3O/PKbqgDUehgSQ17LjgcNnfOwlFidkgagR2FoxhdYZA5TKQv8+up03eKSUpEbWNzE7fe8Tqp0XZzZ+R4MYw69+orst100kYayk/dNQKGTdiIheI2llpD75fmsTHfcMeduHzuDJo7NU0QkS2xXvzc6+C0x7OEBov7aq60820xdGBtHGrLa7Cu24PP3jCNe97xbgyaTWxcPa/fsuecAVCR0DGuqti23lvNSpssK2lA0mudYwaaIm26r0HsXJnLB//+vxso6lAmOwT7Jhsttv4uAiJ3+lj7Z1eJRtAzMMVjldFiCK/2npzhrTOjxsEqc+axLwWHfULMKzfu+nU33+HYb1uY8Onb7lSIxpZdro+lwi6cPydIlU6aqVNbHMX10VB+jEQYioQecoSOAfjceNedWDpzFvWdHfMxvADBivt3SUu249wshB13tW6pYkvnkshh2IVrQ/YRVTjIurIEb/7692ix15bPSdjOnLHjLWNnhjDp7G3vrhRahfehWuecGF/d2EVc7DA7ETnIdHzm47+XMDgfSv34PyfmaZF0UhzPf/RmMxa4CfHSronuAj6ZvImdOGelqqPJVAdfO+A1doEWX9CrxMkaqovsZ6f63va6N2Nnh2yMLlbX1rD/4GEcPHgE7caO4mpRfns9XL50CVubm+Kgx3LwOgQ4RlI/5liJTOiHoclPdDVObXP9LTdj+dJlMWnIXo0+M+HHBIEhTvIbuWxxGq6r6NGCeZM+Cz0t2WSwM88USeMt73gPeu021pfOCjc4f+6MLbZ7/+FjKKtHAfFW3LbBDGJVqYo2kB9O5+FmNCaK45hTn/rb31EMUSyzH7j5nYb5+jmY0TpSYZLtCd5InQ7Ey7JSHCMKGL2YixkQbOw07QS/VrAzQ3p1Yg6rJxw2NcnN4vSdr8fm5roQI+5sxuF33/1GtOm5wjQQr7G8dEU7W2fZOu891DMfSrsjcHkXKIVSLqD8W4BJR05cg621DaytXFFPEiFRHFsY9TFnVnVZrloDHYxdZ6cGBbRsjeN3Y347S6SHDO5953vEe1+7fEaLfe7Mq4rVJf5+T/lI1ppAOL11d6TZMc0YZA3RrLxvfKzVa6KRz/7D7wsuDXqNUYqNVmyOWCBj9tCjzkTqG8qdGylOs7k6scZzmrb7DR5VViv8Al8AMUIlheYV6+jBqCbVzn4TVtdW1FNlbXUV3d4Q97zlbei22KbROvJz0VZXVnHl8mVRbCOc0iLpQBpXoe4oUXeF+jaBsNEJ8k2l0Wy38cd/9Ee4++7bsY+JDR8bif969miU4/6KnWoQjFwzcdG3xZJAMbN+JFMQHYnLI4Ove8f7MOh2sXLpqxLKC+fOGiHSVf04UBU5i5G/4AUOfA+F3tg2u5z34BGYtkwj9bl//OPXhF6jvp8uwRZnGjFg1NGXUpqN8yzNSVMxgSNmYZ/ouQZyZuc8ewStE+fNhpla2z1wLVpPJEkGt73uDeKNE3VaW1tDu9XHvfe9HT0S6nqsDrHFXt/YwJWLl1R/TafFMl9GJjTeuFdwqurFgJAwLyNAiAxTb8BnThaBlK44dYahu332tG8cZ2k70M/T8uOVAjnUCX0yJxae2nvjUBrqoQze+Pb3Ydjt4erFl2VzL104PypTskNndzsvhUmKbBvVeFCYAwCIsNds9Wtp0akHPv3HCZvEcbEikRF2wj5odjeAjlGHP8XGpto5SOFkyrCYBiDqFUcbSfKVMTMzoZN6vM5bu+s1xQnWYJZlwjfedieuXFkSAZF9vtge+g1vfosQNMba8fCbW1u4dO78qLOhjd+gzXhZZskmWlThcC69gI4cPOLyjCgsRy0RN36dkn3m8UYyJeLqEOZY9N1FlTfgHrlpDyvCsMZ4pC7TQXvj13Nn97B66ava0ctXlrxvmrFr4npxX9G8YiMyeRKaw9GeCNMsNIOyfqbKE6Q+88n/mZi63T2OgWzQkPgIAeiI6Wxt503HJNruND0tD9CPNLJF9ERJADY6dshaPlscGWrcvGe1+VANOFROdN0Nt+DKlcsiGjJe5K3uuvtNKp9ts10jGZnDIXY2t7C0tKTF3t0NnJTdHSV17tWRHKfxvmynh1Dy93TqZA+9twq/l9fL8NLHGyf0CGuIvqD+jCYg9j9UXYAsdhSym0hWtaQzeP1b3y2zd/XCS3LKrl694nQwW2gzpbsHxIiE4EWAHOO42tZ9RjlFrzVztFBj/cw//BFnWotkDEmLcUOiaHPU6DVtao7F+uqsMmYDxxeetczRRYg2kLHsru0O6lOoNNMXcRC7YlI/gJ1O2613vh6XLp5XcbmOccxkcdfdb7Z+afXaCPAgAHLxwsXRafajSXK0xjQNPK7AAAAgAElEQVSvh0puasxb9zg7doUgVMMR5Pw4SCP8OfBvPytr5MCS+KB22t5wncczSSgClTQCR+z8kXBwsQG84b73Soiunrf4+tKli6MTl0zQrKCB9xcnnKiemxRGH6G2Y6FDsEJj8hoSCP578B8/nNhxjP7gzh6hNx8XEgDiKpHzF2dHMakfGoEDVmd890AD4YrEF+fT4j+2prSzSEjmkzepigqj5cSk5PMl3HT6Nly8eAbNWl0IGXfg9TfdgcpkVa24wtPk37mzFYo4C3bX8x1pcn0TDiHVdnw+nMj4uxweXyA70NVACk+YasxU9zIjDIc8XtdZ2wolY0fSNHT8aAr7tKAdJX2ETeL1971P110+94IW++LF82aHw79RGOzZRvWIsYPkLTHz2ub7Sj2PHEKzmnHagFDSz//TR/ycdPPiVJ3IAckxsA5CmhTufH719GE81CiTNLbIeix3vJi14e6WpvAMWZgIo0BZmYyFDLsxOG32DTedxoWLBDi27RhmAi8Ts7jpphuxvbkyMjU8Punc2bPujVvYGBy0sFcGUY6Lnjkv2oVj7SflTwgxtL9FoY5Br6aZI4YOkmOobd4rMoYyYd7VP7xyhXBuhzWSYYJjN9yJ+YUFLJ99XkJx6dIFT8zsEkkS1xaMDKKq1Ha9JX9Cc4+bFX3v8xtRTurBf/qI5mA8WcBBy5UXROdsEpEIqZbd4Pvp8qPdYS6It0o2BIfgCr/GGV0kPASiEzF2TJCpmzghwHb88eMnFFY98MBnMD8zrf7m7V4a3/QvvxU7G1clkRScdqOJJ554VIsklE/OmSNebqujowHllTnvXZ/EBCBsXxAwKBzWsM6OUQqKFT+vfi2+ix3NlyCrSCKQNkcIzY8wGrOcRO+faioshfmD1+DosWuwfJYdKmpYY6gpLWKJFUszO1FEWDjPzbYiC/V1k7Aa0STmdmS7vcFQYA2pLz34vxJzauyhTUpt0qRu2GBdyQlzZlQ3xPeN8dQIpqhk1h0fE9rd3t4SHnVGcI/WVVnYwlDdcX/aTd6/1ezgwsWLytpkSK0Z9lBvDfHP3vcvtLPpuHCR2IjvySfI8DAVqSOYvSWnhMpNk7xgn6jY/fKmvdWlhWzWuzvUfbBrHdUd/T52EcMqdV3gSSd8U2g+PxMkujSquTZbcuq4rOixDmTKU7iLIea5M1psljqNvH47RNPGz8+Lym3FDPaKGF5++2ixw2FmOXAwSCTsX37of8lmW7Yodl4U5zP+cFBE9un/a+vanuuurvM+siXLsrk4zTMdGAghJc0Y22BjoLSZ5rl56kuf+tfkodP/oy+ZydBppkmAkkkoNrbBKdB2aOMB27JsS7Isy/iiy+l8t73XUdEM2JaOfpe9117Xb31LXYzxtLvTwR4pSR9LgEZeVpvIk5QJtIYnSxJVoAiPCgRAGTpVePBnQizc79H2pJ1+/e32zb11xtpsf3n8qF358ss+WSdIVpLteGFyvWrBs9Gx1QzLEJWYoCejJ1QnF0gDa19LpQHqjKhFJoxQa288TyHYI0pGTcI0abtzi+3Ea6+3m1f+pz14uNlu375pG68hOVhPcdqonJo1wXvt0kGTyQ1zlMRifHEtAgP/+MN3kgrhZuGHkB580V4nVu2D1nSxWD8qy8zI1O53tZh/opU2C0nPO2AFfxbJfKjG/Sc8JkA8prHvc+2Vk2dZDHn0OM342+3alSs97MgIKJ7ylAvLCU6uoJuqMgVQalnjmkZYpU2W5jGO3oyI1GY9RamedAnPKBgBlgQAYrQBrquDMNd2JofaqTNvtLWrVwiWYHrYqNVoGBZhzHmukM5OngfohMUh19f+qCAUT57ZynO/+wWRKnFociFCiJ3qRFYLtyAQwOq8k7LtG8fESlBX4QYt2u6nt5kSywXWwpBxCKrTIAeeOEnQjG1VgmeunX7zr1gQQC8TrgPM981ry4ImdfuVCYBKZgw5hC0WsIGLY3oLLbBKrqlmqZ/NiFW/p+RTAh5SWaP6ugaqmwpsu/7tqlfSpTxYmKh+qJ149S0WQkDTvbGx3hEv40gNkASzcp6AoEepYazVuvMe3XYnawc1HrTJCFdU4406pdfZbbRjYdNAUkpt63Pao0T4kvbMueIGFqpBXYstG2SmJicpFFZgrPAAMOq99FyvvfmXpKcAVQe5UnYet6t/RNVoh/9WGFeRMlrsLB7Xx+YJz8AowA9dVTun7iH37Rx6pgNFjQOmS7gV/BHWA3TiVD8Y3j7u1zeIc7vAMgVth3U92E6++jaZHzfvrfNkax9k4uJYZk1xVX6vqGrlPGBf5LDFXPR7JtV7/sN/0TmK+q07ZueAC+1eLv1dthsnAMNJ1K9tUJ5TlXJsaj6nPJ3Zi4C9Vi+YHERsR8hnnLB3rK/TFOfxe6Cu/s53ScRD4va97bb89dV27x7w5KMql7q2RiaBv7Q8g/8aAVdoOODFiU6kqFyT90LSJynwJPoeJUfOjeiD2uwxO2Wp0Y3yReDRo8x55s2ftDsr19rdzVX2d3HsYuaTs4xc0rV9/Sv2L1UwPKfEQLG6BtoEmzf5+KNfWhvY1ibD5FOZE231L3XI/8+Rfjqgh8R0OhlyukAGD3uM6TScqxVbvSdmhJKnV8HERQeGPSyJJvGhaBfCxbz1wlI7eeo1MiHTmWq7beXqdQLzMk1eWkm7O4odKXJhBomotjnAVKatV+jkUIVpSAyPFMbAjqzNkkJNbE2CeY+TyGQAMjoZuqy5W/DEVeAgwufAQjvz5l+3zdvLbXVtpd0Bu7OdUzw7ng8jq6kNSvGoh4LVfyrIWWpVb3YO8uTiuV8RSox4MN7zrPxLavIL6c5E7hoLMsKA2d9KzMffcy4XQkfaSrSpGqCYe8bOzXrII3VL5KYF6e79x+3tH/+EuC1K8nSPNB5Qgdg2fTYmQCpdXrQ96V6lEkVHHDloCWgBYMz43LGHnPGl9ClOTNS3snWKh5FnZ77dzh7Sy2Ql3tPAG8wCwbVFSARPQA4UNvPlk2fb1vptjuVYX7vFe0k51CaMsgeZQNBDMK19F+p9Cgx97TzhF8//2o19Q8fFfZcS1qnqm20Ok3SI7BcQCcDYJHrDO2itfaiGOzaGuz2ocJbgaSAAsy+pxj1+z2kSXH9j61F78y9+3DZuL8s32ttt6+vrbR1jLayZ9LzJHThvwFh40Fv2iCK8KHZ8sAEsBvnm2EBQhuTa+X719mkryc6gUcbpfcv6wCuI40n8gEGIWOOXT73RtlZvtdXby+3uxpr6203Bid8H71miADwLINQcBxFHLQ0Y2WQntKANuHbOo0w+Pvcr48a1oYq2ZSP6ifZb4nvzC0JW5gTq1CTcGDavxsg4DVBlcsaCWvUm2rusmiD935BUeLOS2O5Cte2duXbi1TNtA6dgD1TVjQD61bVbXaYZYbg2YQnqJ7UKKN5JVJcgBhCsadaxlKgpdBTIQYKZcq4SStKOEh/6AbbjIBzQ9TAZQAT5aYHSlaft+6+cbvfvrLW1G1fbPYApe11cCS4Wh+y0Yj16+jNxvN86BzJ/ZjGgzum/fPrJ+/TGe87XKiRqNb8QFYV226ouqtrdpz1mBCI2T+p1oCFHBDAECCafaUerUiRzmFjh3E7QcB1qr5w63TbXV0lnhc1GVeyOwxY9B3qzTBvhWLg/X46odsZwXyWElFoc5EGs1ZcCDXVdSrbOlxPznjCOZV4lQsgOYZydfADhzxi5USUJRPjD195o32zcabevf9XubK5zs3ELMkfVAbR+NojIE08cJeKOJU+/x7etP01BiAAvXvgNN5ujkKIyi0cH0Bq+hG5UjRpf8H2wAbFR+3PN/Ey3s2Mel2J6PVbCL17fTkw2qsezOiszNeLJ3lw7ceYNOmRomwEVFurda+urM2FXMnYUqHjLAe7vW5nkxvPtekq0L9Ze7DEDoTxoLsBtLt61aB8mobxW1G5GfDLxEu44ok1R25cX/4MfneD1bl77st0hnQgcOCFMD3pONvYmpLYH5kWwHy2SZ0a/WOJ/ijsPixIstNkXzv96mrSe0p0eG8GN1WXYQOAZzIEWIc/dL+i71RM/CgujlDjgsb6uM3bJPwe5mQpVct2Kaw2AJHFKa6+cPkuqRoyMPAjH78GDtrJyvTtMqqPbZsXw+zlzOpMAyp8Jl7KIPZal0+I0qHMC1BzklgFJkNPNwIQDaMdcuzppoImY2vSJls4ZAEccoOdefJk+wvWv/ov1akQ2nLyEWjbsL4afu0NEiS3BrWhanOaWMI5iiEJJ5eO7N/7Jxfd6R8jMD913NfqmZgvwcLoYI6ePiDnzCnbDyRWqcn96tGqB5Md1kmvHpU5zCHPTXMeOyvmF9uLLJ4hU2drc4MlGFm7l5o2OF0tdW0I3SADY2xVOb6NjcjK6SQkg0smLaAVqtzQxWoDU8eFChVU5N3TG+ZTDJg2pJoqOI2tz7cixYxza9tX//ne7ufw1JxbSbNmHSpIIDpmG2TSSDsATUIg6Uqj0j+LQGrZMDBCe8dNL70+hluSAqBdbR9Y+kRMgWNioA0gKOwVdyYEdQsNfWlajgns4ZUjTQFoWtegFzKbIRimRoahN4Q2+xEwoTTO/+FT7/kvfaxvra+yUQBsQ+LWHRrFtdMIoaVTxgkeQMJoYU4+GY1nbd6qmx6IKqKiig/B64z26AHf1OTQaPoj2KHGrylZn+Pt0Z9ouf/FF+5uf/rTduHalXfz9b9t3jj3J+QfJjDG9y5aoxmgGIEgWeTxsjvjBRDhss7b/Yx9BDt+0Tf5w+QPS1ygLlLgl+12a9N0JghoqnAJwimUze2xpG8GUnoefiUZaeCxtYkIi60Z6uqlj25O1vOm6Dv8ywdaFvftb2+21s2fb2q3raqnZ2WnLN67xwYW8CdiwJhZ1/yAyldQaoEQKMdWkCzelb6tv/AgKVE0y5EfCaEfSCy7BVP9XNXFxqOqTra7ebh988G/t5PGX2xLYEiDkOLEGIdAEGlARcGgQrorHkdUDH5oig9Tgtd6mOMPJ5oPkQlalLKCzJQeDxlE8iJ2NLRinI7ZbiyeV5nRy/xMbqhYVLXYqO/SwS3IAzxLkClUZF1D57uScITo725N2/NSr7fbNa4T34HpQ4xAOaJioZIQq1AxpKS7v5yBToQz5VTCkVJuTtJqyqCqQpA5dHUuxUth/KSldLHFKwqoejnC2JksYpcB32d0207JnDXAtlQxi+AZ1jfEW2zucQwZoFt6LnSPBCYDwxxXL6lDOL5joCKFXjZmT1sTi4SEB36WtsXTizxj8bEZ+P6FSTz06hNCNh6qUDRd0SDEkXtQUlS6Q8HeceZMwZdYXBEA/Ovn6W+3m8lVgSLlRt26taHE8CObbMoI5BTFVaEmqz68WWzk2KnP63YkBB4/aYqfPBOYMX0ySlNJjDVsxIE8lysIeGJw8b6TcNZJO0n6D37xGBLTNHALPxXArspklQDO2s0NOuHtb95iKZqOCexnhXzFE+8OnH/Bk9w2HNDlbJVumJvpsthIk+jyrRQnF0ozmPHPQL0mpjkoQZosM1TnrIOhfeDC8PPovgi6hSvToIjiNsIEnz7xF/jEAnHEfqPEsdGL5qPP4EdFYET5ojapOa7go10WFGt6fm6PWpkQuNDJOzECFIudO79ydKGSz8xcFLSFpcQiUANq24zjajqMxs+manKCnjXCR/RkEufb6EYKCkpSQMnKrqYjDeWXZbJbnAhEuD8JeLmdw6oZn07PxgiHLaWHzuGdcRp0GKEBuEoP60BbcwwID6HU9WbugJ9FZwhAE6plqEz+bbz9CL9gaxkI+pucKB024OYdp6QFmbV5NinjAePhpeNMzJKmihnvNDpFGUZSQaESCykDHTfrcLJxId7pogfU93Pewiz5xDHNAcmDI6eJ5nMPZt0BZ02WdsjXSXhJysTS5X85FFDhyqk62Ptpicuniu+JUsXwn5qZnTika5bO8XCQuajwbSu1g+yhbaT0SRKUXVQkUdW0yBjX0iPAbniAFD5wGCRI3jIYKRNdcIWgP+sGfnyAPORiI8LV8Q0R1GuCq6hKEjjPLYJON6aID4znaCZ34bwq7bDcWcjbRkky6kiEJtxiuWhBjfxlaudFR3Z9qicY6UXNgpMbhxe608eCkJ67jzmd5YeL8cfMOmDQXc1p69+hen9pbBQN/R6jKwfCXPv5N3qKoKpXWuHnGnOUEx7mQsyUvOw5RVB3SfLAb8sQ1mTYmS6xC4u5OD1QnZvP1gv4Erhz8pVWNcnQkVOP0QHvm+Re4qWBTwtfNWyukn6A3ySxWAAvyVtP7VHFawZlhpHIydTpxo5iT5E5MQ9VG4CvXe48qm0yiT5WRPemw7KwUtuOBQDEK4LFOAqn4OEVtx9xWf6mPniZ0GcIoAYxGpq2HULDEabWU2LFWpTicmV8KnZhata2m09BbXUZlDJ/FaKI0ApL7k4wOJTwxL3naUxcwjQf5ZJ9u3BEErBpBLCRIQiqGRm2+PfEn323PPvccqSTxhRInrscMAMD729tkG8LG0dPmu3gRDaiP/dVwtREbd3SttRP+LSEbBQ8+OzabuYKR/lVUEpNh6k5DruCvJFNY07Cxw0Go5ARjU+P9x//JhufgAcwoBy5Jd534oZm0T5MLH/0rq1483oVdIBs/c+xl2fqm8WYHNMwktQWcZHCNcpSEpYs5Yo5zkMqW4GhhUapDe5EqOQbtO5QJCyEhSsjWOXTDS2AMIRrjTp89S55OfA+c33BQOILJbI1KWcqRxL2hbSKgSiIp0zcSOXIKs8AAEEbFwjT1EK33sMthGrWV8W69JOq05nAexeeuTXOiaF9KF9eMNoWwc/18GPJs+TlOblXz6XaJj9A10acX3p0KYTEQFUmu0AmxPY8nrGFPQwTojZY4mZOBZtKecnIY6/qUZL7IiKPtnTvMgfCgiiU7rWIB1ZDVssp9ILcDWO9UW13RlN6Nu6tkEEJ2j+zDYPhzxSxISy2iMk4anrrN7s2kN9PrhQWiEBotk/KmzMFgYooDV52umLeo/ZiebDYrab16WMD9xdPucbK/V0NevAM2P/kJYO/w/ELhylzVCCsagDabF+bpHl2JSONFv4v1aFRRdDId4xkpCjyV0psD6Ie/0zFQykhT64o9g4MWPDeegW4ZhrK5vpzSphZ+FDUEPFTv2Cuvnmkr167y5e5uronczYkdqjE3K8ZZVNyMcBJOHGrSek+ke/GFgkpMC+7BU4TnOuAikWktYeOl9r35hjhp2BycOxs/x+3MetnJ1MFBfludKTBP7Et3eKf9MG0XES0DRcRN5vQDHM5RtIr2JC22U8JB4cSBnpz78JeKswtTLz3yvZEZktrTw0hy8AAOLQy3ibSl8Wx42cp88TTCMwTkx4uEFRmqBpkSXR+4NQmF79VhROJbSYQA7rXjp063G1e/5qJt3d8gYgVCxdKsNUV6oiPhym0btEBEKhZdqBipSxHQJ2rgOAr3VGX+p5Aoo3Ajpw68brovpBFrgPdmehmzxgszFKpcMS34LBNYKSfjul1/SqBSWuY77Gl2N67fSXNc3NFUxZiWcXhpsy9+/B6LnWH94xksqqOnMp33jqOGFB4+BqaeWdugGVgKbVBnvt+WOO9aJzfM/iwPTveYhMClU8+G972I4kSHEkNbiJlQEjq0x/bOtJ0+c7bdurHMzQH98vr6Gm12TwyRqQnZJRHEQjUne8dqUkh7Jgca5lknjGKumc6oHDe0KjOGR1vSA00TTn93PO+0HkOYMVtLGyikqPyA0e0Slatr6oTCvMmpVVwvhKlgVPiKiYRgwy/Suks4a7TUEy5WL9xoCEnd7NjQ/FCGXW4lZAWSGbUGT5eDUuz49MDeN8DpTBtwVEzKopmDOUhwR4GCqp+w370+sD2AgIAIEepx8+cW2osv/Vm7uyZ2QHCRX7++zDHInNG5s026aPGaisRWeX45atgcYsvIqCBHM0PQsanyDVwx8nShhGVDaOVgIfqginU+H825+uwBhoP4PLBkAQlkrSEQ2fCUhKN2c/BynWQy8X1om5rBjOfdVbYrez22Z+jFk63TkpvGkajA9rSuYlIffh7JlIqEIKiYEs8RN+8xcWcDVp4Ym4CXxwMDyYm5GrhGkitwsLiAbmLTiXHNuKMolZR55pnnid7cxcjG7Yft9q1bYmBIWLgLFWlqjU5eo9HJQXsQLmQikRAJcBNcIOEkQA+HBSgCwgh4b4bajd5ybW6yWlgLCCiETHkJYMWlIdI8iaQLGvmjqnFtrgNO9UzBTodOZkbTCuTfKIGEZ4BpwM+zrvHQuwBks2OL8+ewJw6H7IFCF3Ni3WGoZn2JamR4h5HIJF6wcHHgEo7lMwT68T/E0wovSKVpcLwkVlkraJP8nDXi6bQdXnq6PX3saRK9ovEdDhoHssGjNEpDmkWxKE6HpuSJ7opwXla0RPADqUtrUJxJOnT22IMQSVO9FlKsSAk3Ewfn5NHj3xZB3UxBCNqyF5ZS6gUEWQPl2CJtxAvuo9hfMXRYDpPLx/tRU1mYoE0gBKHepM934fy7PY5KPJYTJifdRZJCCSkPO2KnP6v6CF1HBCcaItAibeDwvOvvihpT6UyoRhVCNB4i92WSBO2rjx+3g4eOtGf/9Fm2Au3ubLfVdbQEyfFDEoV14eku2RHiiCoxInADrquKuatXCBMJbHQPd6g4IVydiK5kt6zm5YXvtsXDmlVK/8CtuVgH2VRdm3l+1w5U+VPuQRnFsZZsP8JweAsl1gyjkbG+bFAwVGvUuZXNSddJNDQTM0hqZbOTcYlKr3ajH+GGmRaa5BrpRYkwdk1ORkhsArcdUJ44cvlcEgVJFQZUgJ9jQznv2qMaBpOCFTrGP8LxObjQXnjuhba6uiLmgqt/5IJT4OLFp5l9H/BwRssYANE99vCrOvkD3nD9TJtBzWGzpbDQwm+kT0LKqNfkGhA2xbGSI6vWXmUItykETASlrm6wJwWyx+HGFITN2Y2QMHS91h60ivMkPGBffPbvU0gWbqzyn9R0Xjqbig2A5xwg/0gc2GlzrjdqpSaEEuPGS8y196dgByugVGPgSLGjSSRQLbtmjVLn8eMnCDaEqn3n5//UfvjS8/LaCb5YEG2XB7+HmUGU13a+vE9Y8NFtOcq+FE6nP4n/DkOzt5hajuXLAtLs3RwqCPW0rFOyma3dq2k6QqpVu7ukE81mMJo1BIkPWKNSviH7ldw6NWlICwsMmg5aJDXNbPhw3H1me6aN9ihtMREAOQAmijfAQGHUKEAkNSoEptCQ+BPCFQdCp1d4ctko3XMmGgj0Ju01ZleEnf/nd95pZ86cbv/4Dz9rf/93f9sWD8+3xUOLnB8GbxueNuNSsCog/jVlCEMbb3TQKR0IWPq7uA1u8Y0GDL02n7Hi0p0jTZMFO1fpvLoNyZzobAVWQbiXJ5N3p6oHHYjbh2nWDJcCQzPeGeu4uLRkLZsSrBy43vi/73RPLl14b1pZimJ/ZZMVf2MjOLBlH8mNPlP6hVPJ8bG+u3G3PfX0U7LplHrFhUlyKMQTLzgkP6paDs8YDRmTEuHA1VSSVC/1Y87sRBPhw3ZwihLnNz7JiIkftKUlTNgB7xlCL/V7YeKuSAKM9nSbrwo26ekOl5uydez88OmjlvJ7xjbG58m/eZ0219bW1zgkhtqFhRiphK6u4/OUHEc1p3aKmJRK0Yoh3aNHjCggvNG0iumFQuUhKpypk0sX3p9ubm4yoTCcrlrBksUeIL0JHSV41wn6ZcNjmwPzGaBD2ShVYSCRrF512g6hNdNWo8+FL3WEY0m8xF/garFeiGQDxiIjiy3BTCZqfjIhXgsoEKxv4lRQXfPkmesFz/fNN1vMpYcbpfssLKjITmcqQA6CwBpKM6eDJQjcVEa6s1vmqGSjKRRutpDGEeZOTJFpNRoeU54pthtTgZL8GTBuJ19szyM0vBc2OxL57U6ZbiZ77hFNpeEbkqVwJCeieucSfgLj+u8rohWFpuJu5ZI9ycBCoSyXwQ8u0EcYR5Sga89hlBHnj+gLagxOk3LvimnxBRN3//5WO3xoUaB7xPHz8+3QPOLgbaVQd7XoOAAYldSnHIw17/6M1kOFHsKDwEQcjHotItG+ptgj4j/AhHDqMMeD/kkn1TPmb6YWoG5PxuNYN8dPoAUPlmCsDZ5JPDShCoFJo4N2+ZPf9s3GpmdTojKrg5bNrp57PNrYOth2Zc6GdqAtBidocN8Zv5S5GS44xGEj1bJDF9zTfaSdB1Q+geJ7OVomk7U9xKhGxZdqm03SvWYI8bzppWIee6IRj/MW3m67HSaBxTDpzhyO8RwqicYBlUPmvHRYD0ImaEh2h3V11gph/ygwKI6Y3A4nPp8VocCgueRmylPrzA7adIV9cFjjNPJk/8fl302JPCzzr5SEGHTGRajlWboPORs9q/5lnxlzLqonKaceJy1pPZ40Oyg1BOLfozatQUgQU8hsc7+Mn8pmRwPd37rfjhw9qkEpHuGgbNkA62Xj6Yi6GY+x+67CIWwe1b5LuECSJgYGGPLOnY127Nix/2f6IgjQz2n4i9qWdhnVO4aedvwQdiE7FzPFOFzODu8xYGI2qRMBMzmG8cA8w9T8Lip5iXhkFg4wvp98eumDGXxCbHNOeAXwRwhy2hmse2J8atjZCHnYvU6mGZmeZ8Eih73zOEP99+yJ8h7FAcLCQ+UlYpAfIMHqwuZ5liNe1/35Lv4c1X3meblJT8+g08HMFNbYyBPlx3MPwZ8hCIFSJSunRFBoJvX5/VqxC2k89jIlKbZ1HAZBmxSDay112jXgHZ+7t7nJwg5VPFuD9sQV68YFnHx8v5c6ocbjIWsBRzEdL5qXIpDPbSfDSYqNnG2pqfYDf8c1qhbQQBi03oxMnDzYQTyjQHH4CBRyjDGiFtImI5SS1BvAaK4xLBJ6v2BSxvuMal7i+TwTFjNdILDdMDlhJkz7boQ6WMpJKI8AAAdhSURBVHeFTPM9/Rqn7SGm2TLZokWOZ87nJ3wJFTxtWl2TCMY4SHD8nO9wf7g6QhVbU70/gokKBbj8VZk1NxaWfAk1xOXLv5/SPhtaEw6x2G+l8gZTQiQvdrtWYvAgyYpF3UeAcpry0hEYwXoH9kzJj9mxilGfta0X8SbOrainFL5xRkhaVL0IQbf0Re8/l6DqkMlOjAVPn5g1aY+5NQmIGss4M5qJEPO5g0MaT8UTrB9ULNYFEUzleckzVXufE571iTnVeqpfLHYYzI442VwXLazv6VYuv2tMwOSzzz7iZsvDEyYq3mtuPLJiY6pMNjvqvnrrWqJxklIQiGpXCJbWnrGxuSayXimPytFTokYxcwowOfXwgBH/Aq9u4rze751JQGFuHAmfoDxiampdOUmdYQORFxdiFT8TJaZBfGFWNudKjbBy7RD+5tBwhBRNgRJSWQtBqPT90cwY7nIsqPP5ps0A4RBKuHpOTQfsozhKQ2OHlGGz8eHqqWbzUz8epzykqFC5QY1kY7Upo+gxWoaG/R/9xFGvtQ5bncR45ji5meKjk5ci/igYxPGSWgRXqVOdTswM4cvfIoiBGAffpsORcIr3Mxl+/02364hFQdGLBFuqM4DGrBlMFd5V5rACE3WvmkmMd5/3UM1cdfZ68GifbVblAMuRC0NEogL+jgs+9Ds+//xc51SpH0p5MKiObE6kKDndqp5rPbyq8bHE+lskOLadoUahg8qmj2sPxCfGIIhZUClQePxaCBPjwvbbYQmNNq6TGrJSkE7d+lQmWRLnbzhW0tUiBxi5+pz4qn6x2XHWlMMPBNgJmd4TDm4ZIV5qwTo2/969LQpGZ2xy/h73TBkzZgIags7XnCpd1T/oG02NZ8QrNjtSk1NWN50pOvdJMzXKAWUhtk0hAY1pGBAumqmqKbJww2kbZdMqEJHq2PiYAZkQJVeGV6xTgRQu0SX2/BGC4GVUsx5hTH+GjGvEe6BZgfPHFCb2cMvJnzwP/qQ69vgFePO5djZoqOtBWJDTCUEJiie16W9zziJAua+c2j2GeEAE6T2Vas7BgBMatNDsgTKYz45sYvfJF1+cFw9anddRSlYjoaHm+AhGbJaVeMc/V6ejhh9V6rT4aQ0a6jhCNpw6lDrdb+wifjYuzxsBVSZPSQdWoAwqYJxpZ4mkcalU5cSYKuvBw4fUEuRutIOVEI4LzchE+Paoea/GjI8Th2q/TzLUveJkkcQP9RxBzmZn8/P9CBQg1keOLLloFKbkUaHTvjjTZh5Xric88//8XDZbLrw+GDWkgsUgcmNhxMWOvExV9yqciAqK0GSX2YT+UP6bed2OIEHixm1GrhvHo8c1hkerNtZasKnhHTZDi2xwIBGv0DI6BQinDh9eGsCA7n8Hj65wCM+IpEo2O2iQnETew5oDahYLOBoAM21wIGarxqwaLhmxmouoMbjWAKp+ND5mPaJpIgSgBHvyyaOMtSHJ/YAZCxw7zh1WnA0vT433mT2ZBIqw0XoBVprc+hNtkOZb/Vt56H5Dj3msKoZ22JmsEepI3qr5iGceCR8/F2xoVqWbu6yGHkUooRJRi0fOLoBJBR8WPlflWBErPK54huQa8g7yA8yYmNGI1hJxxMhs6CRLTqScqoH/jg+E90h0UgWY4bCLRtV5zufzp1S6+VFNeAAPPbTfSSbxmZFBq55xJEc4LcGH5GVrI0EAQ8fEpzbSmbId1zDcV2bQtVfWwQL5d+gngCiJk7V/w7UnmQ44xk50zeLwUvH0MDNYhEMkiEOodJA0mouHl8hJokze6GGTf+DZIrPGr2cBq9kQkFBCzejezmWEPJue39H1k6cfEYUEwKEVhxBopHUEJEIg1a4GSp1wMSly0KyjBX7fh4BTfQEgdXMh9hICMJMujWRp4VVPjuufF+nqPjXYzgIgz5WntcTY+G74TmP0qTWcqWMt24akdk7GpkvCR9twTnwWJPY/mw2nJeqf82bNTMgcOMuhYBnU6GcszsEF0UzVzc6192ukaBeZORMRWJtFSCMEw2fQy+XfEhTXsn0N2nN7/DtZF/8shy+Ck/tqr9CSrGIINS8STNCsPjwo+vJQhEwAanxspLzrYMJif+Nc4PuCz6rmTKkMrpr5ZJUsuTlWCTOJd6vW1H5xX5QZM1YqKjtOVcITLeAgxgkvSxy54cmbiNbsDTwnlPgQ9nlSoPlX8axy2NCgGF6xkf2iBpvF8/YTHRUPXtCcQDx3nLrYeTbulRFMSHAwDGQXrUqwOKXEoO3stKWjRzsQQSHfWMH8HUxK7D1zFm/A39y9KenyaGlV3Kmlocbria6OQiS7OkuxPbKD8F71QJ1+0r9E25yGP6u8uvFU/24zDYlrdVjiE6g47+S+a+PDdAxgdU5U7CliWXB2Yqgc4LoLwHujros6d6V4dmGB7feO1SNssPOY5Y2vsXnjpPJeU+H3EhYpATL4YhB/R4j7oeImSVvBK4eNX1wQ5psACg+hjQboPlCiJm72nAbYl0oe7TS+7/73fRjI9n85OQ8T7wFtAwAAAABJRU5ErkJggg==">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -573,7 +594,13 @@
     <xdr:ext cx="304800" cy="304800"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="AutoShape 8" descr="data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAH4AAACpCAYAAADtGIkfAAAgAElEQVR4Xoy9B5xkZZU+/NxbuarzdE9ghmECQ85REBQURER0EcOiIobVNbCGxV1Zlb9gWHPcNaC7ZteAeV0TuigrigTJGSaHzqm64q177/d7nvO+1TXjhq+VX/d0V9269z3vSc95znmDeM8v0iBXBPIFdLIV5MpHQl9paN//l6+p6Qn84qYb8fh0C/ONCHESIE6AqN1BHMdot9tI2hHSJMHfvuBsTE9PYcOGQxBkAoRpVt8DAGEYIpfLIo4TRFEbaQoEQaD/0jTVf/yZX9lsBplMFu12S6/zd2l/D9BqNTE0NKT3RFEH/HUripDJZPQzX5MkMVqtNjKZUNfgNYMgRBxFyOfzem8ul0MnjpDV++xT2lEbhXxePydJ0l2ZJOH92bWrCwsYHBxEgtieIYXWIghD7NyxA+vWrdP7/LNpqZEgRYQw5WcFuq+7H92JL/7oN4iRQavdRJQESHkdvp43zXtAqPsIwoz9Lg20hvy8OE3sd0kHnVYdmRR4/TlrsGHzIShmQwSd3T9Lg3wJcaEfmf71CDH8/1vwSGPc9F+/wV1b92GiGqERUeApkjhFq9XSwqdRB5kwwNUveZoWh/cSRTEenmjhqIMKKOQLXaF4IXMhuRm8wCmYTifWElEI2awJXgtoa6DXc9GiKNLfC4WCNh5/1+509Bn+q9PpIAxto/jP4PspeL6Oi1kqlbRBHn74IQwODWHVylW6Lu+hdyPaz3avS0tVlApF/RxmA91Txv2N10y4iXs2DBckoYJELQk+ifgwKTpJipmFRWzdtRdxkMFCE/jDn+7DUjOVUP3GS4MM78Z9PpAm/HsCrh+3kjYcYsSthhTwjecdjPUb16GUzyFo7fx5GlQGkR1ZiQSjyCQVJNSKNEQm5NI0uL1thdMiEPI7F8BWvV6r4ds//TkeH6+hHrURdfiB1LZI/4UIkEljvPXF5yFjSotWs45H907hsINWI05iLTQXmQu2YsUKUDBczGazgUKhqAWnJdDu5mJJw/zC2kW9heDDNptNXWdpaUmay/fZxuB/QCehZYm618tns3p/o9FAuVzWzybkRNeQ5gQBqtUq5mZntaEP3XIo+vv69DfejwkgQODuLUk67r6cNtIGJAnSBJifn9dreW96T5ggE4bI5mzT8TPnFmt4+PHtKA8MYs/EHAJa5CTA7Xc/iKUm7UkHtJeUU5gmiCmrGIhiW0d+ju4rTZC0KcMUf/XkMRx+xCbk+drFvb9Pk2I/qs0YhTiDXHMJmaSJfK6KrKxHKjMVZFPE5RFkBs+QMJfVLcUvf30jbn1sHLO1lsx9p5NIeFqUToww6eDvXnweb1M3045byCY5IJcijrzJ5AImKBaLWlgKkAvDf/dqqjf5XtDalE7j+Z2fy+sMDAxIUDTdFDq3MDfP0lJNz5TPF2SVKGhqJc0rtYXfqfVmIRJtBm+WeV95aovbQP5e+Ll8favdRl5uqI1s1txDQK2UVTBLwbXhpvPmWvcWxLrHMEy10WdmZvD49p1otGNkiyXsGp9F3GohXwTma21Umxk8+NhWtOIYowPDWDM6gHse2wagiKhjG5pOkMrEfyNqydS//IxRHH3sYcjRDV3zgY+klUoFU1NTyKQBchmglC9goD+LF55/LIbzixJ8JsigU8gju/J8hCltdtC1s61OHf/ybzdgz3yMatsEyC9qHn/OJAmuvuxp2Ll3L7Zt3YrNmzfioDVrzBXQLIY0uSZe+vp220wuzTW/+Jo4AIpJqof1LoEbI5PLaYNMTU3KHVTKJUTtSIKnkVpcXESYzWgD+c1CM9hstmTJKHh/v7wHCl4mmsIPAyzMzyPP+wiARqOJUqko7XdbH7EzqYVsQZvOW7Ukjc2sh1kkaYIwzwfMShHA2CPNIU4jPV8my+vxirYpOnGMhx57FAky+nwa93VrViMMUuwen8DCUoRCuSLXOr57CusPGcbCUoIbb3scsbM0iUx+jDjifXTQhyVcevpBOP7YI5Cjdfra93+cTk5OIZvPYXF2Dq1WHZ1mC83aEi668Ew8ZRMvkKATtVBZuw6obAJwsAu2nLTSGD//9S9x1+PjmKjTZ1mA4bUvm6b4+xedi3sffACDAwOYm52RgLm7qZGjoysUsMnP0i8FAbgZzbS7YCbsIBMtIc1YDOKDuXyxoJ/r9Tqq1UWUSyXEHXMfaWwWhM9GQVNb+RkdBXctFPMFZw32DyYtwMogl8mgVltCJpuRsKn9vGfeEy0X/TEFz/9nwxw6nagr+JSCp6Zn6EZChNkYxSjB1h/+AgPnn4MiN5CWzwJDfiaFVqvVkM/lUGs3MTs7q/UqlQoI6Q6RYseOPRgaGcHs4iJ27NiNeq2N4VWjCKI2vvrLe+UAJHSa+JhrEKPTbmEk38alpx2E4449HJk0QfCOD34kzYQZNFtNLRhVr6+QRy7I4PynHI/jBsaRBDk020sY3rQZcaUf2cxJ7qadEQ5Mw7/89e/gvskFNNsddCLz9RRAFhHeetkzcMedt6Ovrw+7duzEMcccI+HXanUJmQLx36npWgi3CWgRGlOPopx+G8mKd7hg0KL+TC4rTeQmu+22P+KUk09BTjEBfawFiabRAcplBmyJgj0KfqBc0bVCxg30i4r/GEMkev4AKVrtlhbcgsUIWZnkEI12w3Q0yaGDBKWcuRMf/EnwykKyCOlKqNWdNh79yBew+nUv12sz2by0ks/HTfOlL/4Lzj77LKxcOYpyJY9cJq+sIuq0XWzEOCdFua+CyalJHLJ2LRYbEXbu2YeJyVk8vGMav3lwL8K4DoQ5cylUgqiDVaU2XnTWRmzZvB6gqX/Lu96tfddxfpVBRtxsYMuG9TjkkEOwAtM47pAYzVaKVUccDpQqCDIbkIYruhE1nODrrSo+8cUfYu98FREFrwAjQSGu400vfibuvudupTrc0f19/RI0NZWawZ0+NjaKYrHkAjgL5LiQXPBcPo9Mu4qwOOjMv5QQoYvwd+zYidnZGQwPDWPzpk363Hq9oVSNLoAmPJfLY/v2bZhfXER/fz+2bNxk6ZpiAKDdifDJb/wSrX33YsXgEAYH+7VBR8dGkQYBRkZG5AYp+HZswhifGUchl8FAedRlCpa5cHEVIHJzcrMkKZoZoDYxhU6mgAwySNKONhQ3CTfiXXfejqOOOlKbJJ/PoL/Sp+C31WxZzBGYBeOO4vfFhSrmag1MTM4pGJycmMSP/vgomkwL40Qug66FmdWmkSxedPZGrD94NeK4jeA1V70t7fo4mp2UMVeMSy65CFOT0+jEAR579HE866zNOOWofgSFQYSVAoLcJgTpMJIgRqCcn0Jq45Zbb8cPb74X1VaLKaQWYTDTxute+EzUmnVF6ktVi7Z37NiBww8/HIWCBWC9QqcGc+GoEbx2LhMqIOPvvannxmCEzvu/7757sbhYVZ59+mmn6TWNVltWI+lESs8ovPvvu0+awLs9+sgjZL658crlCh7cuQ8f/Pb9uPJpwxgaGMTu3bt0X6vXrMGGTRtldnPZnEy/rpsk+PUTX8KmwnOwbk0/skFemRAjfL6v2WigzRRRAVyAb/3bN7B+06FoNprIFYq63pFHHYn60pI28ezsJFaMjiBIEzA2NHdYQLvTRtzpoES3FobIZ/Nah4WFRSzUm3j0iZ2oVhuoN5r4/UO7MbOUIHJ5fNrpIG5GOPfoEZx34joMDw8giSMEL3/jW1Lmf0p5GNgAGKoU8IJLn4PFhTrjEH3Iw48+imIY4ZXPPQKVTBXIZpDk1yE3cjLSJI8gJKDCuH0JH/rcd7BzugFaKKYTo6UAr7rk6Wi2qIFZmTVqH687NzdrQVmlguFh+m8LvJjSTExMaAE3bNigTKJSKTvfYj6RWkCgghbhN7/5DdasWYMjDj9cWsznec+n78RVf30csi7Fmp6dxbZt2+S7+d7jjz3GNkFAN1DGzp3bsXdqHpkkUrBLa8QgkYIfWbFC1oqWwjIASxt/PfV5bK6eg77RMdTm5pANs9rU3EzNVgsbN2xQlL5z507s2bsX+UJZcU2xVEa+kMehhx6K+lJVlmmxOodyOY8iQSKmtKHhE8wQCsUC6JK56bKZrCxBbamBbbv2YGJmEVGUYGZuHg/smsPjuxgQZtGJmR01iTzh5ecfipMPX60MJqHGv/T1f5MqCGDixwgzAM44+TgcfdTh+NOf7kMUmy9dvWY1JidnMTG1B1f+xVEYqt2PTjNC/3FPQWbkFAQMurjL0EBUn8XVn/oZlhqUfILNa4bx/HNP1s3uZ6eVH0vWWkjmt6NjY2g06hgfn8CePXtw+umnC/EbHRntWgYfnevtYYg/3vZH7Nu3D+vXr8eJJ5wgMyNrkBIPyCKJIgnxlj/8QUIblhkfxNFHHWnoYpxICLV6DVMzM6gtLEqo2VxOm4jBICP7NavXoFwpy6r4lOy+Jx7AVP4OtKt1HDN4EVavXG2pXauFdquFSl+ffvaYAnEOC+kYzWcl8Fp1Ud/n52cQZlJUaJ06bX3G4OAACnlmL4w5LPenJSDwMzk9h30T01hqJVhcrGF8cgq3P7wLaVBEGrcw2D+ING6inM/gvFPWY/3YANI4EpoXvPi1b0gVfSaxfEIuCHDB08/C6NAQaswj832YmJzA1MQEVq1cqZ3M6PySsw7HxuqvcfBp5wLZPLKrTgXKa5nEIY2X8MjjM/j4N25Gp5PijKNW45xTjrHgURmmhyzNT/svRvaz83PSKm4ELiDTNAaAK0dHLUVzUK5/D9Gr399yCwYG++X3DtuyRWkU79NchWUY//7vP0EUd1Cv1zDYP4CnPOUpyiYoeCKJDPwWFxcU+XNDcSP4qJt4ALV21SoKNZR18HDw4vwCwlIOeRCCphu2TdeOLYAsl/oUv/B9yjSE5Pn9bz8060tKjaNmA5kcIe+m5FEp5DA6MqwUVprPjZjNal0InO0dn8DiUh3bd41jZmZOIE0rTvDYIw+jkxIW5/qmmJlbxBuveC5WDPUjAP1vB8FLXnsl41kkxMi5C9MYFzz9yRjs68PIyoPw3e//BzZs2IhDN29CjYjS3Bymp/ZhamoGpx67BRcdsYS+0RGkURbZkTUIhtfL58edFn5ww0+wYwY49YQTsfagtUhSQqghgh7s3YMjFBQfqMHswqVhtADUFP5+zSoPmdqiefDE49U/+tEP8OxnPxv5XFYC88ieoYIJvvWtb6HWaMjMjgwN41nPehYKhZwEz6zANhtNo48tLLjsBYxmZmdRKpYk+IWFeW20pVYN/YVBBGmbS4rQSbUZtXXtSrlProvXYXyTybEWYICPNF/+nJrM7AIIMwSRAqFrvH4hl0Olr4yQbq3TkQvqRJHwiUa7hXY7xsTMLDpxCjrq3Xt2Y+v2HXh8zzxajRAnHbcF//mHu3DVZWdhzdgIQOyAgn/xq/86ZSrD3cE8cmSwgjNOPVFARTabx969M7jngYfR11/BYYceqhvs6yvj8ccex/S+Pdi0biVe+pQKiuWKHqCZFtC3+kiAaU4c4QvfugWnn36StJU5pfd/HrmSBXA4O39eqFZdsGXQKYMvoW8Cd3LL5qHnJ+HXjJwd2KN0zL2Wf7vpppvw2GOPKTikmTzuuOOwZcsW9Pf3KY1lbYGL3GzWXexBvD/X3aCG1IUuj7eoPopalm5mrEbA/6TRLjefXZiXxq8YGtFmaneIT1hsYM/sN1WAbIbWKVQAawheiDyBtEIO5WIBhUoRGVqiqI09u3ejVmtYLYM+P8xgYWlJiCQ3RL3Zxt7xSXzz5/diurpEDBdRJ8FVzz0MGzYejBzRUwr+Ra96dUp/YVqS4JgjDsWmQw6SqcvnCgizBfz+1rtRb9RQUjCyCZVyUbs+G7SRaczj2KE9GB4cRJhnKpZFFORRXrEJIQpYbLewb5GbyBbS4NP9v3o1a3xy0upVSYKxsTEtpNA9p+W9xRvTGHst/feTzzijK4ReTb355pu18ShcCpzvocaMrliJhx95GIcddqhuiJAufa3/UnlC92z+la7QinCEf1vaXNS6YqHgAB3TYH72vfc/jF07d+Jp55wrX01s3XCJ5Y3iP4eCp0JRcQw5zCAfpig6wRcrRYT5HJJ2C1sffxyZXEHK4HEAru327dsFz/J384s1XPtPN6Da7iCKAuTTCK89fz0OPWIL8gqeawhe/TdvTGlOozhCmMQ46fijEMcRWq7QsXbtwSoQ0Fc1G3Xcc89d2gAEYsaGB3F05hEUC8BA/wDy5SKCXB5BNod6M8Dw6AYEuT5MN/Nox3l0gixCpEKOzF57HIi733zgdR/5uNIyBmMffc81KBWLLnWCgJCudXDYAS/zuc9dj5e//Ar5P7+JPOwqH9qkSWzJT1NYvHeLzjN44RWvxre+8gUhY9RMvzFlkVTBo3ZyMwQy3VbetZ/9a7278huR36uNJv54+20487TT9Fr/5QtNvJ6hkgmymUSCzGWySv0YzdNjlfM5rXWhUkCmkEentqQUOFfIo9mIUHHPkMmwfgCMj09qA9JFvulD30A7YqU0QSbo4BXnrMfhmw9W4Kilv/B5z025GOvWrlVAcfDa1ejvryh9mp2bRZxE6BCISc2sEKTsL1eUfo0M9ePQ1h0Y6K8oTy6UiwhzRJtyCIoVtNopBobXIghLePvHb8DehTb+8tLn4vgjN5omOcxbwhKgkeA1b/8AOiHTwgD/dPWVCAPnHhJfj/eVQds8fMhf//o/8bznXaJrMrWzwoyle94ieKEIPnUC5ee+7K+vxJev/2cBLMTK9xOig1It9bCSrxe2TwO9Zel1XYK4EeC+B+7HkVu2KENYtnQs1tiuN+g3RiFv0XpWpjsE91kuG0jwMvXlAggQRPUlaXa1XsPw0KiCPX6x8ENwaXpmBq1mW3HYWz78TTRbHcRRG/l8gsvPXodNB6/D8KALkJ/z/EvTgcE+HLppA4rFAlaODQk0YJCkuncUK9qtLi65Wm+iXDKfy2NkcAibc7sxEFRRYP7JSleGwVUWGZZTcwV00gwKfSMIikO4/LrvoFGrIwlYnkww2NePjetW44Lzn4Yth6zDJ6//Mh7dPQ7kCtoI1175SgyVgLjREkKnyJZAKgkU4H1VMbhiGPNzCxjq7/szF+Kj+t4/eEFp6VPgjf/w//Cpj7wfiCPVnVi4sYoagSl7J7+FQQatqOW0ny9nqhjYexwxQ9kRU9ogRKsd4Ikd2+Q2ezV++V6MEEIrUypmtFnzJEi4cnM+E5hlLRaQKxPCjtGq1bFt+3ZkCzlQy5tNuqYsgjCLUqmCMJNDNpfFtq3b8I4PfQHVdgYED1fkU1xw8lqs33AQBomM8tkvu+Kl6dp1q7FuzRoMDvQpcFMli/wOmjWmBQxsmg3ML8wrNWm1Y5nKfBhg3Wg/VlbvRLaYRblS0aLxBmju+RC5Yh+QZJAvD2O82Ye//8x/oBU1EGYI+ph5lwYSnQpyAjYCFm8yKY5auwrFTIJmdQnPe9bTtdkCvjYT4t0f+xz27NmNv7jwAlx0wTnIWu7lavWe1cPCiVUAewUuoVNoCPG17/8HfnrLHei0G8jEEforZRxzxGY8/aln47CN683KxTHe+9FP4pqr3uSw9VAFIC6gIfIGTfOzmOb9/k/34f7Hd+D8M5+EjesZpyxXLL3lYebCzUXLUSnnpGw5MpPCjKGY2UD5e4WxVoUwbQeNpSoeeuRhlPv6FHizFkJLiyCHThRjaHgEYdYRWDJZdBAik3Z0j1a0S5D4MvGr/+av0vUHr8f61atlvivlfJd+ZP7NLsSImNt7sbqoaJVwJMuEQ5UK1jbuRCYXWuUqzzwzQMjiX5hBm/VUokhBHmvWH4of/G4r/uO27dpYbW4qMEJuW82fhZT+QcGwjNL5+7hZQ9xuId9ewrVvfS1ymQI+/vkv4eFd4+4+aWEiHLpuFd706ivQV3CEiwTohFZmpZCotywtKyf2QSECXPPxz2PP1Jxpdmo0MRIzGGN0WE7lrbCQggBf/uS7tUlrrOk7nMCTKch5EXMoCfHCt7xL5eIrX/YSrBstY3Z6BgN9BdUuKIRGo4Xdu8exa/dOvPB5F2KgXEahyHWzjIHxbzEXopjPolzIIlcqIUg6aDWXcN999yNXLiIT5pB1sVcmVxGoVF2qyn1QcbmpGezJUjIY9eCZMznB31z1uvToo47C6NCIBJ/PmW/0VS2PmXMn+jIq38uSIdOf1cEsGrvuwPCKYb2n1N8H1qLDIMekFDFyKBT7URwYQTbH2AG47ut/xI5FFnEIJpgtJZbA6DTPYM5CeTFWmAlk00Rwbzlp4bCDBvGH+7eDdLFcPsccVItJGJiVqDBu4Z1vfT0OWTmCX9z8R9x88+3YO79g1y8W0CYvkFS0NEGGcUsh362tJ6nxANBuyVfyXgnEEOPnfeTiOlqdWEAUOQkK1LKM6Gm1DIXMs9LJIkyWVTWWsyNRusJOAykrZtT0hG4kRSZMcP27r8Lw0ADyBa45sX76+ACFLE19TqhbtmAaPzW5TzB2QjdQLIPgVS5bRCZrha35+TndA91th7uMMQq5BdmsXJLnMcgCXv3Ov01POP4E9A/0qUzpmSI+L2XgoAjZ8ceIGQ8OjSDMpajNTCC751YsTe+WyeEN5ooFpAysuG2zBWRyZWRyJYT5MoqlfoRhFnGYw1VfuAW1CLpBCo4mnOaOJsyDebwHkidZQ0ijlrFhWGpkvuwCIZp9sktYcTKwhiRP4u+GS/B31A5FzTkSOwzdEsMna+VfQruMri11C7nGiNp1wdc0xdyE/EyRJDr2OX4RubAiXDhCYTZfVArMjED3w43SInBl+TtfqwJP3AFD5X++5rUYGBg03oDz8Uzr8rkMSrksysUssvmsyBSsMywsVeWCc7miaFf86L6hYQWM5CNQu8WFSN3n0fX2pNDdNPcfP/Cu9Oijj0bfQAVFLnpgCJonUdCP6I3coSI65rBipB/ZzhxytX2IOouo7duL6clxjK0cQ4YFCNa9aSZzXARWxXISfC5fRqFAn5TBTKeED33vbrFd6Q2I8qt2DeKelrrJF4fmn5NO0y28ESy4g1ms4AMGcYo0dsGW6E0mSNYJjD3kijq5vOruZAGrPiC+Gz8nNMzesWnQiUU8YZbD12nzOOSMfpkBmQiNciEeRXS8O2U+WQQutYxliex++NncuAS2WDEMgwSf+ofXYHhkRByCbM7cFO+3kM9K8KWC/Z4b7oEHHkA7jkX+LJcHuDgqjBl7LUB1adEwEJZkewTfi5P4+w2++rXr01WrV4vlwaqV1ziCFdqhpOrStBGhCjMkD2HjaFu8vGa9jrjdRNysYs9jD2JguB8ZmuACNZ10JQYreaRBCWE2L7+XLw0gn+tDjDZ+c/du/OC+mvBjZlOMSOlDpXUUvMyhOSWaRgrn0IP6sXXfEpKQ6R+lZygYo3wKRCogjXRsU2k8HTWZKYzWtR+M/0ZPyOditcuBWKxokc2ijeBJoEnarfi1Wg0XD9iG7AaOzl0pLuKzhgy+YrRbNbMQ3Ci0KjT9LuAM0wiffsdfYWCgT4hhzmt8wOAui3whlLknqBS12rjznrtQHuzH4OCQTDyYriZAo93R91p9SXEXuX9MSRhBJQ5V7Kad+n2A4Mc/+U5KQCOXz4hkwN3vH0j+nTCj427HaQfFxm5k2nPYsPEQRMSK63VE7Rr2Pf4QKgMVJEEWBW5ZMkizOSAoSvgQm4QBSQkD/YMIM+TlRPjkz7Zh20wTqk7QVwZMVag1zu+H1CQgK9Od4NzjNuC3D+xyTGBHLdZdG3tIbF2nkWTL2LMAMS1DYAJmakaBRdwkjCXSZZKmuAmuTE36uEyzYyZRGXRtugrHCtbN9RSaqIXc+Lwjlpup8ZaimZknN5/aLvgaMT76lpeif8BKtdzkSlkp+FwW+XwokkcumxEWQB4e01fB3glzfqDFmCXOY3qpij2zc5iYmRNPj7WCyZlFTE3PaN2EzjLnT0l3zyC48Vc/Tum3izkLSLxv5wsZFPDqeQoOQH3mUQwkS4iSNhb2PobDjzsJcZpFVF/Avom9QGkE+8IxzHcsKm52OjK7LIIwJ+bNczGYEkqzyRlfrKoQwyCKpVLyyK3yFWL16tWCbVetWiWK0Y7tE2i3UmTDMgiRkGxA16SFdSVaU2fXTOCid5pDWS9uD2/JaBIpdPpD+VwK1Qo6PjXzDFlqqzYV1yS0ErIIoO493WvyNY73T+toG8SII8IFGE+0m+b34wh92Rj/+IbLMDRQUVWQ68/r5sIApTwFTnOfU7DXaNZw74MPYcXQCmT7BjDZifGr/7odv/j5r7CwuKh7bjZaiq083Zv3q/RQjSP2DFIoupxb/vDrlB9AOpQ3W3yDSrREk/IFFLIhGgsz6M83sDQzjrSzhKWp3WB4Mrn6RDyydwaTM7NYmJ4WLNpqkDHCsqpl1wGjJUdOZIzAxgOqCYMaMlomJicRODIGF4qfS0TO4EvL9WnGy+VB9I0MYGx0NTYefgRWrdmARx7eiUZEDJ3mXi0SXcFzc7HkaigZwRZWDU1oKrSoGhd3N4AyBLo2x67hhvELpss6gEaBo29scBU2a6rgpjMLqTuReTerwcIIf8fYQTy4pIOV/UW84xUXm+ALRgRlbJPNBMrj89kcClTGDNCoV/HYvgmMHH0qrv+3b+Kmn/wUzaUakpibqS16FtNgGnLdpweedE1bG/8l2Pu2229OuSuIEgmWJFWnY61D9LnFfBHtZhXlPJDEVTSJ4i1MYms8jDu27sbM9CTI0m3WG8rzSXpQaZJa6FKIgCkSF5sgBzlkDeuCUTqmbhLyAai9xgX3xAziBTSBSptUuOH9RdIkslsYMwyvXIGD1q3H0aeciU6SwfT0IoKYKZsBJGCwaF5N2YMv+lBI0liCMNRALprzvd02JII0PW1cerFr6uBr+JV4eM9bFwnb/KhF/wbskC9HgXdY/ubnJh0cubYff/OXF6GvUjIGsKvO0UUJwMmhtTQAACAASURBVMnS7zM/A+qDa/GjO+/Ad7/4RSxOT6M6tyRhE71jzKB7UZxhULDhLz2Bp3sOX/0L/njbzSkrcTmmR2J0UvAdVYoYZbcaTRy0ZhSt9hLSxhyqrQQ/fGQntj7+BHbu2KViDh8iH2bRYTWo1VavF4kN9CX+i5pLIERmNKILMHap98Eyxu5GuVA+q+DfvQYyWOli4u5B+HTtVhv5QgnDB43h8GOPw4bNR2PX3mmkCWlGXATD9wn3d3NZ19JkqRU1uCPfq9cR/OFiOizBP4OYSq5nwN+HzwR8XYBK7zeUrbxzEdlQkCvXlqkc1+ysI1fiZRefp3o7LS7jWaGdxEyyxO/p5/OYHjgIn//eDbjlxz9WQN1qNlBfaqJea1hmwazF1ROM9r1MF19Wc2cRfX3k97felAouDPkhbDeyBgfGZwsLCzh43TraAbSjOqr1Or53z0N47MGHsG96EvW5qpkR+lpqRxoKsFhYnFckOjRozYsKimxFtC1ljrgBGEGLlNhCqVDosm60GZyvtZ1sixfzvU6jFMn3PCT3GO89E2aRKRVxzMkn4fjTnopHH92joE60aaVUbocpTTOzTpaQNmTbCBPmmy1OULDnzCbvn7IkV4GsIAV+jlhpG8HKjbpfFzjK1MsCpOqGMaoXsYEEr3j2GTjz6E2oVAhG5RWRM0dnUpvPBsrfp4fX4Gs//BF+8Z1v63lb1RqYWSxVG0g6ZlloKUzY5t+9lRKwxKyFn66mFXNxMvW33/m7VACNfEtGwdxAqYJGbQnDI/2Wr6YdAS3fvO123HHbXZidmUCtWrWOGknGkSmcxs7PzWgB+ojiuQVQlbOnGdIvKv9OCJMwr1AnSlDWzW7UUDHv5ykkBkl6TMtZXb+sqMxOQ/3DFQf7cNqZT8bw6i0Yn6wJE0ji5cWhn+X1fDCXOFPPq1PjPa/fkD7g4tMOw3Aphxt++wCa7Eejm0jNaoWsx9HfuoYNWgLhDS4IzKYBWu2aijtJRFcX4W1XXIzD1q1EX39ZcY1RpcgoNnpVe916fOM3v8F3P/tZ1BaqhgoyaK7VQeNET8brdxtCVX1ZFrA2rCd8sMdOWY6hecG2HQ+nytPNXuDxJ57A0YcfoXowIUxT1A4e2LMLN/z2Fuza+oTo0Z1WJLSNC5QLrSDDYExtU0xX2EjhCjVSBEGvy3mPj4yJhjEIpPb5WrUE3omF5JnGEZQx7bTXE41yLdRsfHAVLW/GTUUNDczm81ixcgVOOvNszNbLruHTbyrfsGnBIz/TbzSfx1twB1TyKT74mmcp335g6y58/IbfWZSeWPA0UExx9tGbMTg0ALJvdkzXcPeje9FJXJFILeANtJsNVQJzYYLrXvd8rBoZRH9f2bh0LgilArI28rXHHsO3P3s9gnobs9UF631okyzJFJNt07auXmFo0cTjd7QuAW8eCEnNTbJ2IcewbeuDMn584F27t+PILWSjLGtbSsJDp4Mv/e5W3PmnP2FpsYrFuVlpL1E9+TYX6PhArN1q6Ca5YqwZq0ecrcmwuEFsWxclCxGLY3HLuNhWwrTAiF/LdW+XirkHUBqnaot1wfhWKh9t+9hAGiQwpIC1h23E5iPOxkw1Ul4fKge21IqWjXi/zGVkm4zBqQI0JHjds0/BiUdsEMBF3ttbPvNTcQUOO2gIVz7/PAz0FY1k4hDHWr2O93zlF3hk15Q2ra4dR4rASW8uFXO47lUXqWuGtHFDLRkQk4oVYm5sNf7hfe/B1ONPoF5toLG4hEg0MWtKZdm6G++4YpoXfJeswt/njJwiM2+9WsaDePSRe9K5+XmsX7MGCCx/FnTioMqApcMgwAd+8GPsfvwJzM3MoN2oi03q4dzeHnANFiCCRi3nYjKQ4W5nBymBA0er9bvS/5uoIXljZMowyzDs3ARP7fZt5f6BfdVQ+DbNGbn0Dnvw1/RWhdaHPpQo0Nia1TjhjAswOWtAjG16mnWn9Ywj4tRtVFcoCgNc9+Iz0NdP1GxYz/APn/gOLnv2Kdi4akiVSNKoSZfig6saFkW48iNfxu6ZljYPg150Wog7LP7EKJWL+H8vvxCrVq2Uj1ddnSRMRuO5DH40OYWvffjDyKUhlhZrmJ+ZU3Acta0TNqZ/d5aOz6D18B7Qde/qn+x/cJCzBG/BAIId2+53Pt7Ff0w7HFNUQUkSoBp38I7PfwFRvan8ul23smTiWpx1QZcoehCIQmfpVakSc2kGLs6HEV4VE0abzOWdaqNqSPs8iMRqYLPe7sKdPupXHaDXnCk1dJvK5azd6N3FCXzkTDY0GHRwAOdc9Jd4YjvhYm4qq6AJ+KHQ9R/dHwXPew9w7UvPRH9lQIUUami7k8itsXTKz+qrlJV6Gb0a4iy88rp/xXStZe1EHSvwsGWZ3/vKeVz3hhdibGRIVVG5L7c+gysPwT/dehN+8JnP6P6qMwtoLbHjJ2PDHshWcmml4hkH0BizyBWaHALLTKZbZHOMJHEHd+14kFVHV6PmbjI/4YVPwd83PYWPff5fZY7n5+ZkchTYREZGoKaxYCKBqJKX0YL5luGUwxKSjh7MdhzfZ2M7WEnTZ6n6xc+3yNkHcHFkkasEaVmquXBXePGbRDEhNcBPvnCsV6/9phXcIHI4GFq1CqefdwG2b20gn83gnGMPkRn/7n/dxZKhLayvwgXAu192FsrFigRPIVHgCgLZxMh6OmOOuC0XwveOT8/gTf/8E3EXhAa2WNjpICVyl3YwUAxx7etfqALNgOfOuecc2nQMPvbv38RP/vXLlAZm9hHgksd1LsjRz3rmAsiUZ4ysaWtlcDV9vA98icR2K5+7dz6QygcIraLf7MV4yBMP8YddO3D9176h/LK2uIimIw9GrUj1cC6l0DUKm4tSKNrCEaZkBCn/Sf5XR68hN73XHHOz1KqkdrnUR8iYE7KCq9AKHMs7Qu/3voubVQ/sQRS3v2je/UQMml5x113vO987vGoYz3nui5GPs3jSYSsxumIIP7nlQfz89ifkl3NphNEVfQg6EV777FPEFciRaCJuQkEAlPAOdSDF6sSp1uoWOacpds/U8Jnv/Qbjc0TW2GjSRqfFGT8RBgvAu15Hwa/A0EC/TcfgtqcVXHsoXnf1mzG5fatKzlN7JtHh3IGOwcm+zNoVLhXJTwhxZFDx7DXQwp7ZK7JiCf6egtcOcRUkXwZ1ayfB/+qhB/HV730fGbJLG03l96VyWRE/YUMPanAgAS9M02XRsHWMdtqRmjFs8gQrgMbn4xdNF+MC+kDW232TJFXarsF766mC9RAlfflYZt5tPrZNd+MIEhBcOsWF55qqGOKsAu3Ohk3r8fn3XgeNYBChsw0aeQFMCjzbyDgcgDV1wxCdFWIwB7aBM8hNMTXJoQVVDV/Khnm0GzU8MVnFxFwTESNql3qxBFUuhDjs4DH10omHILIlkC2vwOLAClzygov07/pCFZ1mB20Ol2p7opdLZl1G42XmgzplG07wHAph7CbPHbQAO9i9/T4J3hcTlArqhYa6Maj/z4fux5e/+31ZBX6xyCL+eQx1frL/2uBJE1CxaItLTp5cAtOwTgdlNxjIm+dljSWJoGpUoR6Dw3TQz74hgdP8mQV9rO759mb/wIpJnCWggBmWW3rJoIj0Lr4vRSFfthjFggYce8KR+Ke3/r3VFBw6YN9tuJBCHocRMCAkoqaRCMp1m/pMVtHsy+BpFmvkXlzM0VvA6xZKHIrm75vSKY1swV21GVz5ssvlPmenpsCCe6tJi2kVSJE/3CaSiXdarfV0d2FO2PrzFN84S2DE0RDBrm33plbNMTOrFwtbtxunlm+dmsK7r79eo7zYfz49Pa0LksMWkbNOPyZcm5W1SIKXRlOQbvAAr1UgEcL5TW9R+JnUdGo+f2Z0T7fAtmUjL/ohRRYjdWnTLK0q1bL7VZroNibzYFW6OP6M07ESG8ZEU88qPI2z0kg+tWvHPvPME/G+173WWQubKME14OcRMeyicc6dMDKXSVfjlJl2GzbkNjvDFlcA8trWGzQ7jnVXG7VJMgWs2nQyfrvrYVzzt29WlD89OUX+F9qiSpu785u7m7Y5KrndiOvqcZiAXusKNZIZ14qbYPsTfzJT74TufYU3lwRdluIYV33sY9izaw9WjKyQORNAE2bEvo3qNk7MI2Z5ES4ziv797zTPxhcvyHdj2ZIkxowVaRrNpjB3sk206TizjTmcQ798dcsTNdQz59I3+XE/G8fh1EqpOJPGaYcWSUkE0zZHRhC1i6VMoNzfhysuex4uOpkNJS6ecOsiDXVAUrfjV1mLzQEy6Hg59LTgys3qcTvcv6Z7bTapOqSQm0XBbHkEJ552IX744O342LXv0maan5xGu2Fz+biBvUWWn3cWdVmbrTZgf7PmjO5XYAJn3CNTv/WxO/aL5gwNNRaMNgHBlzCDN33ww9ixcyf6Kn1inwqQcflqa8nmyfmgg2wer/FKP8IQfUxZAvpO02JW/riYziIKtrWCg2kaF0OQqcMCLE0xbdKmFI3bNpt2tcP0lwNEe61gaPc3EiK50RgzeOugZgfahlwGI6uGcd0rL8eqsgE3VoFzNWz304EIoyeKShP3Z2Toc+lQ7AeLDZQ1+c3gt0vQUUo2sPpobDzyqfjmrb/CZz/0QY1dmZ+YRrvZURWOFsBruy7hNJ2/M/KKZWTmEi2GkrZrjay+z79L45949Pb9BO/RnS7+y3AmCXHVJz+FHTt2mUA5k6bRQKlYUdNhxFzbTYOU5udC5IJQ06fYj81FZMrDpkBGwuz0ILmQr1XFS926ie1q23eiIkuPxKaxFE/+TNQsg2xlrknRJj6uoYVu0uMBdCNR8Xt64nxFjUGnf5+lPMARJxyGa156ETLUSEfA6DXRvaQLm79nFT1vgnutp35nXG5Xo3d7wAWtXY/sovK1R12MFasPwse/+Gn88IeMqYD5ySkkkbVs+U3vYyMGsvwitd1vCG/apRgug/EKwPsVY5iA138neAV33RZhUpECXPu5f8EjW7dK4H0D/TKRHkWrL9ZMu5wPCYwnpfStVMx3aT/lkk2x5AJzwyzn2AGWFmwciEG1ROIsImcngP8d8XTjsftq1HKRpGsJnDb5a+vhGR73jEZl4YJfrTpHlbQVRKnuEDeRLZbxgueci+c96ThZGwWBPdMovUXxwv4/v7Ms263ULTd2UOhe8N4qHHfmy9AulvDcv3yumjKrC1UsTs+ps9lrhH8uWVjH2OFoWD+mrbsONPU9FrHL//f4x4GC38+H6Kksgvz6D3+AX91+J/ZNTmPlihER9Kkt1NzZqTkJQ0T+lEOEbKJUg+PHOEdOXaaWRlhbVluRsebcudIqW6v4ZRUxC9i8pgkAcUQNPxOPVoAFE2M1G2BB089Ie7nO76ZfMo5wjFsjaFre6ytwvjpHAbA0zf759771FRjmbDqW5vTN3tNl3hxQl/ea7u/Zm3OBNu4f9gzuOiqp0nbbv/m8p5zzKuyLY1x8yYVI2x3DTJbaypq8Jve6VFpemfWsZVPe11NxVJ4mXOuCX+HzPRhG8PgjtxnE63DcA4M7H93f/8QT+MfPfRb7xqeENDHlZb5OwU5PzMgf2pgOju0IdeP0nTRRjNR9p6lpl6dsW+uxiBcy81bb94vnYwbTKm/q2aded6NOjTxiqZkPZJbnxskMujSG16LwhEp2HL5AUEn4dyR3w0IKcfNGp4VDDzsc1778Ik0IEYfAWQxtHIcNeJN7oHk3VpFx7Lw2+2zGx1tiHYnla7uCKdZJT389djTn8ILnPxedelvZUmOxDgJlPiXrjb+84PkZJlRvqYmeWvpLOSnO6Y5pdXHC/yR4v2M9hZQ6e8Xbr8bknnGR+VeMjarkyKDFplVbfkkiBunCNKNcNM1+4ZQot9i8GU8j5mf48aX8O6vaxBMOFLwewOHntPISpjRcW9YshWRqpeVljTfT6tunVWdz2YgXGrEDVhKXLUyKKG4jzGVw8bPOxAufdCJsAJ4Fe70MnD8TuIJIY+76Qpeyu57ah4tcZOks4+GfmXEkOOWcV2M8buOSSy9Wl+zE7n2qzJHZpC9qdU8rOF2WBW6ub8CGDysG8jELKdi9BTFqvnoi/2/Buy2QBnjde9+L6YlJ1BttteV2Qkb35JSRTsVBBqOYn19AqZRHu97UBAcxWVUAsRiAi0Vs3LTBEEMztQQnyJV3wEi3b8+CPbJNJHAVAARDIAxp1m3OjUYnyGotR/8+4PK+jhrPh+a24ZeqZq6+73237iVuS9Yjq0bxrle+EKP9JBwaC8i7pgNNe9ctuUaGLqPVW9NurOAYPb0ECsZHYQnHn3s5HlgYx2svv1xDlnZyXm2DzRd+MzlAxltnx67pFmnYs+i4CrbZrWdgOZay6p/WsVfwvQHRssZ7wQPXXP85PPjQw4hbxqAt9pUM3NCM+hhjK1eiVquqVZjATnNpSa1V9SUifSZ07ThXRyf6Z40PXviU3XIwxfuhpis3pbhcNUlpXcrJkHy9VarYR+bUwpENliNtmVJqhhtQLCF6mJobxY0oMbCIrNsYaSZALk1wxMlH4e2XPBMJ81ovfJ/f76fJPtbowQDE0LGClFHUjPcvSmRP+sshxtlwJU4454XYWp3Ei1/0fAl+z9YdaNVZOXRkDnLundnWWtBqGBnfSCeCqx3IJUw+g5C9DS7rkOvz6R0F37sjvL/v9a/ezPzyjtvxuS9/w7LTJEFf/6BAEuaM1Wodo2yhyqZi3HYaTTSX6IsLaDc5A4+948s0oS7o4Lhv9PMH+kx7Tw/BkprB4TBuSoVnk0p7e3y8sUwcO8VtBy2My2098GHgi6F/QtkI7XYJl4mme3AcyWUXnY3zTtwiq+ILJb1BXG+6p2v2cvV6wDF/T5aWmpn3eX2mshknPekCPLQ4gZc+7xIRR/bt2IW0nWoEqwJAFyAIqnYceW0gujONRjGkUabd+3xNyzAOo0y8h+T/O8FrZ/QM9vc3vGtiGld/7GNokM+dJOgfHNIN5Esl1JaaSvM42WpmchqDlT40qkuW57rOFAqeXz618IQLQp0+mjeTq080Abvac7cq5SY+9lokWROhaMZt90CP37wezu1uZpfOMeL2kbpZF2sX0+9oxrKhZr2vPmQjPvjaS01QnAbta/zO5HqLpXtydGsfzPXGAQdaUWsGseccXXcqNh5+Kn6382G84YorpNn7du1G2OHQZXYYWVTuhejxerOgoWb6UuNVYXCC1wAoR34xsGx5uNKf5fFeyH8meAVQKV7+9negsdRUF2uhVHInOXCEZoyBgSHBrgnZpBwQmMliaX5hGRNwJUW2QcvvyiVTUNY9Y4vEvWScd+1mZ+L9QtJskg7uLbsXJr/3gjzK9Z2Aeydg9UKdGhQgrGB5uD81nuwWfn6x5Kp7UQcnnnQs3vr8pyFhAEuouMubN+vXjd499O2kvHzfznKpIdQFgT7RC2Ks3fxUrDvkWPzbHf+J9//91UJMJ/ZMIMP5/4504S1ibwbmTbfGonhwxroQDFdx5p9TM2RlnaX5M8F7s3Wg4FVxSoFXvfNd6h1nixRBbqZz9DPs1SItScWWZlssXVbXmrVal51DhZF2OJ/LefDC792pE/74Ea6Zh0u94HtNqyyGI17sf2iApYP+iw0XfA4fsXdNsouC2XBh4IqnYBlvgMEqNy3rBmq7Zg09l8ObLr8Epx++1t7j8IflWMG1TrvY04J5l8FrQ7syc7cBw0f+/FuMw4+/GANjB+Mbt9yIT77rOmVDCzML6gTWejm+nA9Yl92FabH66RwobHgJXSLHprtBEY65a4qSLAd3+5khsTmWmyGW/5bic1//Fm659143FaMtrlkmzxw5oxnsNJXkp7MnnKldwBMZ2k2n4baQojVp5y0f9GP9ZHxI16Xrkbb/5lAkE6blrUyXvNb3+lrNv3flym6q5iZlmbl0ubnKrsuRtoKv0NURHKDE/J7CXrlyJT781iuQURVwmW/vJ2n6dTrQvNt9LWMBFoAsX4P0miNPuRylgWF89LtfxLev/4Lq8NXZqsUVztR3i1yyGm5su+M19Lo1tZ7J3xPSJtBlkT3nBHD+kCJ+H9X3Ct7vpt6gjxuVulptpXjLe9+thgIb/l9ANh9qxh13HevgnAUbtRqqH7Ma3G6Qg+5GjKo/3Z3M4HYhP88iV5q1XuybUzCXaWD+HjXT1VGfeMxIt1DjxqHZ/RsB06dy0pSeYr9lGGZ+fQrpFZQuzUWH1nDBOCWw4connHo8rnnxhSb2nqi+F9b97/L7XsFrI/QIngcRHfekVyLfN4D3f+Oz+P6XvoL6YhW1+bqUwbtf8fnUEk7XbVmO/8+ex9rSLO21vn/OxPGvMSjc4RqPPfzH/blWzkQtw3+2BqoMyc8neOW170Lc7KDW4I0lqPT1axIGT4KgeV+YnUfSbttkKJ2SEGkBPZZPky7SBf/ncHdNvhaH3wSvmXZuSrSgzq4sXErYZdosQ578DAIcytVpDTgqNJsTx603S/Edtt2mDBdc+nEhSiFdKZYLau3ONpuWNunNf/UiPO24TeikjAF8N+z+Gu03wn4Rv13VxTLELXyXTQfHnv1aZEtFvPOTH8BPv3ODMqOleTaX2nxc+3IVU5uNLlqV/u4yCV+UUXOGS/2ISfrfi1vAYhrP1fnfBN/VMHd+mvdb//CJT2DP1JR8PRejUCxr5CajevLp9uzcI+5Kq9HQOTcqtDgN87uXBRdj4jpSINMxtmARPOkhG0gj3YSpZY1f5ot30yEH3XrBy5wTruQGcaNWbJHoIhxh07mTLnjj0tRumCDNdBOtuufoNTE4Oop/uuYNqGTMTRyYvvln7NX85Y3gy7Q9pj6NcNLT/kYW6lNf+wL+5bOfQaNWQ7tu8/a94AlWeRTS8jKL6Ak7+9TWc+q8sBOljL5knopnL9i8V/B+d/aakO5iO43nv+fabbzlPe/TpEvWszmtqTzQJ23rHxjA3p27kXYiDdRv1xvIaEdyopnV5mlNBJa4yF34ucCpZbMuLXcVbvu558uf+uBOiuLDWqmV48eJ6pjfZ27PQoUGASjiNW2zcwNcW3NPV6tcjidhmC7p9dZfZ1VCC/5iHH/8Ubju5RcjzbigqtsHv0xqOdDk27+XBU/6uTZJ3MbJ578RnUwGV13zd7j5t7/B4gzZzHbGzeWXno+DRytYu3Ytthx+sjSf+AnHovArk7cDDLiOkZo3OqJ38/iS6mIVu3btxPjUtNZgdMWIxrsHjz5065+ZehmVnsHCvaaeP9Mkv+Kad0h41PhOJ0D/8KBQqpGRFRjfvU+CZ3GmVeOZZ4ZW+QYGCp5+U8CJS1XsnDTDnHvNI9l/vRG9F7/OaaPA09jGnrkqneBLsW6tVu+jenseG0fSi5z5wMtyca/BDvVzgRWbQvjF2IQ+ts5zdAb68YaXXIInH7vR4fcuqncuwt9nr8n/7wTvLdqJ571eJK7LX/ty7N69ExM7d+tcnA/+w1+jsTSuruX+8iBOOvlctOheOA3bATtqi3R1CmIZhgoukzbM+jlfryyXnTQHCt5H0YEt3oEab4fsxPi7D38M+2bm1KPNHJzjVGTys1nMzM6onMlyIjWe5XCBIq4Y4mqpsgJ21lsGhaLNZ9UZKgfUwL22q+/cgSbGqzNwg0ebLAekPZOhHWDRfWgXqBhGYOe8+SKP105P+jBugINhXVRurdNWziV5k6dPXn/t6zRShfN57b7deXvupn1N35t/g2z5xSPI3FSNNMAZF1yJJhJc8BcXolpbxPzEFJ739NNw7ilHKzvZu3cv2u0ETzvvL2y0W4YFsZY1RSqEtuYILU8P/iHShYO4FfASgeD3/03w+2m94FPpu4KSG/90L7763e+KK+fPNB0cGsYS83Z+eMeIGA1W55x5p6n3QZa5E+ukocayuyTmQAP23HVbq5fNpu+y8ILndcjtY0DpgzSZbwEX1o/HyFb5rzv7zaXConJzg7ISyE3D9/cya/wm8FG+ByIMjLHNEDV5wEEbp55wNN7xmud13ZQ/dsz34nvBd69Jp6TYhtVIA384NvbsZ70ZDXRw3nOfqfR3bnwSV73kAjVu0Idzrs2WLUfisCNONndDy8Jj3kQbk7S1bgKyZLKZvtHF+U3hu3pdJuAF3+vfe4M6X8mSeXQRqRinaYqXvfOdVp1rW55bKQ8Y9ZcTSjkgoVnXMIBC1qL9ZsOgXp9XMxU08gT71SC3wQKy9c7v3z3bTWV08C6DthBhjhg1I1gKuqPhTdQ4agg/Y+P6Q/T7J3bv0nc+QYFM4E4kgKRUKVvzB+/XUbcs6nbDC103Tm8qJmBJPspGnw8OD+Dav30lDls5pJGsjPIP9O0y94Ejk9AySPDGG6DP56HHZz3z9SCP6annPRWduIVocQEvOf9EFDJZNHiKRpzg0r94EZJMCXc99ATufPBe3PfEds0XaqlBdRlml3vTBDHWsK313GIcp/H8+ZEH/7AfEaPrTx2I0xW88416KLczrv70P2Pv7nHU1QiRiK9e4kmPBGg4cG9xHs1qTa1XFHK9VlVaVGBHiqNQ+SmWjI2I+ok73jMU2PPIfV+ZzFo2QKWYRV9fCUdsWounPOVMnHXqUZpLx5YvBWX8X8+YEl7zZzffieu//WNN6uJCsAlSvt2Z5WV83R5wWfPN9xuubwJM3TGqTBU3btmCj7z5cimdhhj3VO+6m8ALvksv94pEjU9x1oWvx2IS4YKLL8D87BQKnQinbFyFUilEK83h4aklVJsctJxBJ43sEAWlecQ+HATuXZvj01tKu4xzCDQLHHT7yAMH5PE96JaChG7o5wbEdcsnwHd++TP85Le/F1onDh1CTa6iH6HpnJ2e0lwZGh+mEJx/y9/zNTTBbe1U46bSzDdaNVWjSOvK02wHGR1Pyu5RNimefczBuOaNL0auWEa22G8bZL9wX2Fo128vM1qXq3V8psvecDWaHfo6etrlnOrLdQAAIABJREFUUyVoxs0aeaH7s++6oY6GBSt9SvxxqHRRCS574bPwgrNP0LHf+wvebWSX71NYxuJxfYc8H69TwbnPfAlum9qFv3rBJToAapAzfJMY2VUrdVgz14vsZimmKw9zvT1NWemby90Va4Dzh/O2Pjxjhz/buA7boA/ff+v+ZdmeAwB6BW94ke0C3TiAxyfGcd2nPt2tvtHskHdXLvcp6FuqLii4o49XvskTpjsWCFr0buNLKBa6DPo6FWs6ETauGcKpRx+FVZkW+ioZTcV68gXnoNTXr5mwYaGvSy1aFsufC94s2DK/3FLDBB/90vdxy+13q7ikESqOmOhNvQWLPqOwdNQqeNZBq0O1dW073rRvbAj/es2bNQv4QMHrda4L2QteZVKXiTQ6/XjqBZdhW20ef/mi56BVb2LLyjE8OrFP1TVyA3RapROumLLi6RlY1T1hROtMZI4HkCyPPekOqGQzhevuleC1XC5a9qdGdjnc3VV1gu+ZlUYm2LWf/5waLSi4Rt3OSunvH5QF0OTLZktNlS7YVGBF/63+OlKtoibWjo1gKBfgyU86Fcds2YSoVdcD7dqxC7XxvTa8MJvBEccfiU2bNyIln8zNxe2mTeLjOwxeW9ohjTpE0U2B8IvvovrPff9G/Ow3v9dG8C7OZgAZ1cprfm/MY0pj7dR+8BCZxwxKTzzpaFz7+svUb2iwrxVgzD0ai4auwCqCdm6u4vvsKpz5lOdgMm7iac94Cvt8sFSr2rkBpYIILzygkCCZGkRczq5Yh/UIxT3ugV3NPpfJWYDrqWou9uJhN9qu/5PgvU9d1qYe8KHH/33qhhtw59332KSodltBUqWfB+GWMD0xhYQDfHnkB4mYmVCb45gth+JVL70Mmw9ejdt+eyNKGaAl2lVq57W1Wf1b0oOPrBhFpZDF/Ow8CuUsTjnhKE3PDDlwWX2qjnPnTpdga7NFuAFml+rYPTGDJ3btwa6du/H4jr1a/MgJNYMQe+d4+JHx69XoofEtHk9YVohebIGLHDUtoGUBhCAWZVmq5PHuv/1rbDhoTFC1xQn+9Gsz+ewgVgbhLAp/Vxk7AkcfdxYerc7geZdchAyVqNUSNsIDhIsDA8gXy1izdr1AnJGVI1ixYrR7uBKHJmkABYmjUUcnWEQ80pTdSY4E09DcnQABEUhO5/CC7+5q59QP6JZ2Zn65YGBPFePGu+7B17//fXWnkBUqfD6bU8co/dLsvgkcdtBKXPv2v0eZGscFcQ2PRPTuuPVmhARIskTAlufMeoKCtKbTckeXt3Dc8UcjIjBT6dO8WBFn2XHSbOBHN96E2+5/RFOz5xc4vIEjWW0fdNpskDDNZuuxPUkWHNPKgMdAneWDE4Q0us1ghxQ57pqbasXOVf7dmK02pqUV1TE0PICvvu9q66qVK3DBoOPiJW76tbFmLfXadPRTMbZ6C+6c3o1XvPRFiBZr0vCxdWtw/AnH45o3vQOtbAGLSRNtXoeHKDLOIOdQQE5TgheLiC4kxz5CK+ho1Bt7DgXKaWqwgu//UfDLhYHl+vay1V8G++ZadXz4X76IfRMz6g8XQ4XDQfI20+bT11yDdSvYnWrvtvzdH/CT4t67b0UhZKQKneaktIqATj4vTIAFHg76L+RCVPpL2LD5YLTSAm689R48uGsvanEbDRI7NayYAmCDpAmEEueu9314nnZERJGLwaEMPJ2Kx4ISG9XwX1f77hZ12AnLmX3uqBYej8b3b39sG2rzi7bAAa/VUimUtfvXvfQv8Mwnn2LxkGsIUUbAymPkOABdMmmKE858Psr9Y3ikMY0rXnwZpsbHsXHzFnzn+i9isDyAxRCYojYrM2B3bIp21EQh5LFsAZpRE40kknvlBGveY7vdtJZwztbNZTVFVKd1c6Q6Q46H7vvDfsGdL10uI077C16+xEnRV6T/8StfxgMPPGoYfKOpAf2CU8MQ737Da3DcxoN79oyVZ81iJLj/3tt12jE5Y9wbGvTnqE9qiswVcffObdg6OYcmkS4e40VtijqIOHyJ6ZXNf3CsXetatSKFaWmxwDHqqYQnxorr+KG14EZbaiyKPqaqHUu+hbyOXtFcHfbQpQl02CCPAUkTneTU3z+EQqmgMXC8xvzUAh668x489tBD6Bvsx1fe93eu/85Gu+hxCbeIim7m3yqgIU4+66XIlSq4c3o7XvXyy9FXqOCmG36CTjaDe2tTmFiYwkJ1CUnU1LNVin06P2igUtZz54KcKQAPbK5VUa0t6dACYhWe/MKAUCdq8339Ayb4/YKXIOmJWLVnl928+6k3g+IDfOTrX8KOfVNYYhM/o/OGjfwuVUpIW21886PvWw4endYbVSrFI/ffaV2jYYDhwiCWwggP7d6N+3ftA6e9WD5uQ5DIfy+VCAtnNJmKJj5fsgHLImW6IUd8vU6iEiOVymzRr6ZDaDqIjUenQDz/j/dLS6Hed3fsyMLCnH6m1WAA55s0+R4e1yZ2TmQmv6/cZ0WifF6t2SPFPE47chPWFAjqOJaP8n8P2bq9n6Z40jlXIFcawKONaVx26aX49fd+gioifPeeW7Bv9x4020ZWpZvUHB1X32DbOT9P5wNx+geha83+56idpmYOCH3V8CgrK9OtqavIC753Vy6nKlbrPfBrP1oRgEen9uKr3/sBduzYY5F1DC1UpVREI47w7fdfi4JGoi9/+c979IE/ycT+6qGHMKHZM/TpHbFMleY5/0QjQ65dsdBnlOwMO3nKBssqYjWfyvr7gU0P2YxtDsKzur6iXYNzaX2kyc70coPZWbBkFBV0BIv8uwNFOFmDMDXblnTEaLVuWLhmJLlBDBqz2gKZBfTJlXweh60exbFrVqLAw/6kOZbOMoA97vRLMTK2FvfM7MSHrrsO1/3j+/GlX/0YtWZDKHwjsvI3mU1SRTe7lm3q/L2OSHcDE2z2OQcgG3pJ39/f168z6Q2Asna2ZcH7kqXPT33x/8+jvP1KpMKtA+CaT38Ke3btpeHRTbTqdRtRlglx1MEH4QNXXWlND1phnuGQw9bJCXzlxp+iqeF/Hevf1rFlxqnTgmesLas6vyDghydcqFhCwZfLNoudqKF65G2gAdeVAmabcRe75sGDPNpEwjZrQ76g+eHlXj3l+SFkJvmz74ilC+Ln8h54f7wWByl3hxvFdlIlf6fqFzLa/DwpQlF8QgIErVAWmw8aw6lrV2GIz1EM0LfqRJxw8tn4rx33497f3or8oavQzmawZ99eo7g166jyUEhWNDXg0CZue1STsuY9ERX1ZW9aAI6Cp1vSc/oBlAzAKfyuqfeIneOieTLhfrNJnML65gCvv2EnxTv/9bOYX1jA7CzPRcloECJbq3gWXV9fP77y3ncgdLXoWpDBh7/2VdQ4NiUb6oiQYp6dtBS0+T0yham97FtX0NbuoJ9DgrKmvS3Oi1NbtO1gTXB2x4F6mhf9Hx9SftpNxTTiAidulG0sunwfq3vmq42Ry7P1LD6Ym511J1waLz+roo65EgqFFoAADg/3NdNvk78ZTXOEO6d1G1hlYA/LKszzmYszRz9qzTqcccTxeMa5z8Efdj+EY9cdii/9/scKPHfuG5eb4eeIE9COxGWk4EV2FW3dOo/ov2klaUH4HDq/p5BDP1FOziEin4BuK3KnZfYKXubCC77Ht/cGdDJSPTVzL/x//+1NuPnuO7F376QO/SHPnmANtY+jxZ9x+ql4yYXn4+a778FP7r5LTY8WgNnid32tZ+BqegPPb8/qYfg1Nz+HFStW6Pw5G49mw5asvNvRYpG5qwEA7nwZ1eXdDHrz3bQgoYY38ShuGzHuJli6oNAPHKBPlabHHeXMS9Vqd3gSNwCFwvIsn4MFG97nAlubq1U7FoSVNzfixRNMbWRMoHHnNKp8xv7KIC48/VyklTwuOP0sfPOOG/HE9m1CKcW2nZ1HvVF3/YghWi2jsrE3kW5LVDNOJGvUVSuxCdaWnjZ9+uh6+voqA0a+3E/wPbTh/yuo289fU1vCEFd/4iNYWKhpGjUVkBOyeAulgQEcvPFgXHjaSfjp7XeI8EfByyfnKNiiLkchtohLZ0JVzTS/3REofSbAYI+WwOY4WRrlhwaYZtu5NLxml11K4Wv+KwVIjbWAVZ29jrTou2jNh7puWneqhI/CuxbB8d1keplpMDPgKRsayWra1p3ooTMAjEfohyiYh7comxuBFUaCUayzX/6Cv8SetIaZ+TnxG7Zu3ar8XE0scYLq3LxNv2KwFxEws1OuRGyRGyNPYXkursrD6mewdjVuECrGsuD/jDpki9OFcntKH12hH3CI3ds/+0k0GhGmpucVPTZqNtRIc2Q3HaJhwjR/vDGdZknBMmcv8EhR81MUCjXMTmCsKHCisBgQSUhu5IiaHbN8COIFLX2n2aW7oK/lG1ivl58OQplgnbjhzJ4f70n3wSDJV+Z4v0pFdUJH3tqomVE4lyKAhNTuXM4CLlLIXYaijdeBzDADRDJ2+Dn8PSNsfbabK8DTJ7wbsvGwsY5Uo5AGDlqJJ537FGzfuk2pGcvNtCzjeyeQNFpoVGvabETl+Kw8a0mhk07T4vApy9U968jGwtrBg1AtweXxCmj8cVVdyrCDGLuTMRzdYZmdIF/TuzE+8fWvYNvEBKrVprB7Tmmy82dC9K8YxvCYnaXOPFrRdKXs8GRrCOC1Cjx1SVagoKofTaHamkJju1aKRQmRm4BmmMGUmgl0Ph5HtFD4oSJdHlIoQTnrQAvgF0QWhgER74dkkBxHtFkwyCyDGtls8v1sTc7oc9hDoPo5aeWlopWRHW9QAx8IALmxo1xs/seBDxQar6l5QI48yvunm2H0L1eSy8taaAN0Yqw6ZB2m5+ew9uB1WGpaUBrX21iam0dSb2tsvHx+HOu93IA2JdQsmT/3zub4s0GEOAnn+TuuwYP3/j61xTlghu2BPt6pucesZQ16ulb473sefwxf/vH31DI9OTGHQr6o1Ee48+AAVh98sB1Nmg3VDcoGDGq0zLNj4vB1FDoXRvmyNCpAlnVoQqSOOSvf6o48UWzSPQrMDiCgNjJgZDWQfycSSC1TuYSU8EpFAxa0UI4M4vv7/WYmMEQLQjfB82vM1Gd1xKgd48n4wE6I4t8NCzALofiGpedm0xpINIPVrAFfTyvjLSqxczWNJrZxma61kxiHHnOEaF08XbJEhm0mr3N2o0ZLhwtatZAwuKdpG+1a13Xt0lZwshGwJjNXabz/7t9Zde4AjfcVq16N9ibeC/9AwXOo39s+8SE0mxEWF8m1ywp21TSMXBajBx2E0dFRTM1OyXxT+NTu4eFhV+hIBXuWSzbtsdJX0QBFLThLkO7kDC8gj35ZfMB0y7c5G8uFAxm8hov5oxOiLGswHpoFexFTsB5yKV/L+6vWaoKhFQsw/qDbopVgOhVzWBOjbaNPSQDq+TOmLgtWtAIUsqhSOm/Oavn6HV2PQxap8Uz1CELxWjOTU+gbHtIZczT9tbkFJM0I84uLQv40ccMxj72LcmLt1hv8rF/rVvIbgefsulnB9931X5pzR43vFayn/nZ/2fPDMqazHAf4zfC2f/4Y6jXOrKPW0RTxBApCjQkqgwMYW7VSJowaNzDQj3KlpIhVJyGHduKjR/WGhgal+eaKLKf2zQKeI0cky1MmqWl2HLdZCk260vwkoiuWHtq1fHRv8YGVNN0UrU6Mpbrl8JoL70AeDwFzc/HavE9/eII0iqddOl9NzNxo2NY7wOfz2D/vheZd13Puocv3Szgh0/n+OMYSz5yhu8uRjt5Gp2F8Bs3+cz32XHc9k6/xusppnLBAQ9DGjZ3pys8Njrr3Tzd3Bd+bpv1fgveVp672uw/+xNe/im3je9FuJViYZ4pT1BgzPiyPHx0ZW4EWz1UNM+Kr0ReroNOJugQNLqhP88zk53XiIjeLD4i48GZuE12b16FGWquz5eMKLFmo0Gxao3Ornq2UyooXFA4hT9LH5LPJSyfzRXPeeVaeTZ82KNfq3/LVDgWTmddxIxaUskjDz5J7IP2cfATm7AUSSjtyORQmT6xmcEaloPnX3D926XJjRG1Zvdm5eRFccwULUvkZjG98u7lMfc9Erl4l9WCZZh264FOm3R2lEtx3501/jsk6qEGvO+Dsdf27p8nwwL/fct+f8L1f/grNRlvCTHQSFGfR1+RnVq5eheHhEdGFS5Ui+ocGFeRRmymkpXpdUCwBlmqVg48NauTf+BrCrjqpmUOVNJ3aOPq95t80gEMMbCqXMSoM6vRQrVqdecx52w4r5rU85GuZQYQGMXIaAyJ7boQqwR9r6ba5fPzZ+2w+o9c+Rur8PWuVokS56ZtKK4k3MHhsNPRMrD5SOAzWuGGZxtWjJtrVpgpdeY0zIx7h5v8fkE15gft2NNERPMXKtZmL2+i+ZAn+J8FbU9//LvgDTQzR3XaY4m0f/QjaLaZACRYXaoJZmWpRUwZHhvXf+Pi4dn+pr4SRlWMStARcLGjB+DN/x8XwttyEb5G3bwsiBs28lILSyVGJ+V47KcOdwuQHIzmki8+loNH7Sofbe3/pDyrQcARC0pEBONwYLHeaqY9ccOioVu6wQglQgRpLp20dHMQgtMh6gMiFlvdzTDsF7wEm4QFRpBm+5CJG1RrWj41hvLooZJM8em5A9e/tJ0TDOnRWgM4vW+4eNsKHa6QgZtAF51IE997xn1aW9RvCHxLYE+Xv5+cFCu2/KbzPd7w+XP1PHxNyR3Ig/X3o2oxo+mmSy30VbQI+RK6YR2WoH6NjY1Ys6aKCnIJdslTLmUlh9K7rlg/P3zP9k5+LLWgSvu9MGzWLx6eyscOKIkaNtrZmi/7FPA1tdoyCMoEthuVz09Gy8JHVu8+TJxrN5dxex4rbgctadDcPT2NgOQeIm4NTudsRSoWi3BTNuoE+BiX7moHO8AlYX8igWmvg3GOOx9bHHkGLlb/hUUxWF9BkZuHaprgpmSlYCuomePAZVX20MSuaKJY4i6nYwUrYstJe8N1u1P9D8JYO7F+qPbCO8++33Iwbf3eLmB6cwVpvttRMuUTggSzb4WFpACtffYMDyBazGBoelpA0BsydskBSJk210jidHr188iMbH0mioKnnmTpK2RxWrTyWgosiuQsiiL5TlwvF8WFWvDEXwE0gi9ED7XKz80RMjVmlptPXu0FNis79MaQy5cu8dS2uAB/bZEL15hYUh2iKSKGoZ6LF8CdcEtvn9TIF+vkYm9eMYSxbxrZdu6U8737b2/CO970fLUcKFQGTpedSHpe/+FLsG9+nieIkYDTbCRaqDdQ7MaqLiwbwaPCT9fzbKBEneEvnTK99D1ovAbFX4/k6f0Cu9+8HCp6HF73tIx9EQ1BigrbTiqjVUV5PXj2FTAtAXln/cJ+IGMLdXQ+4hv0zHaLQchbNKzjiyRAO4aMrkOnvOe+eu52WhP6W9Wqhda58aahcRr/XEaU8Lk3om1kw/T3DyZvU5Mjyap2k6Q4Tcpi+LI8zb0a/srly1GZtnhangwxi5042ctiMAB99cxPpYAaetunm5pn1KiCfy+Ctf/VaHH/EGlz7/z6I6blFNYf84js34PmXX4HxxUWlnzwHgHLaeMgqvPkNV1j/gPy6I7XyKIG2O0/HWciY6SspaHrUAMG9t/0qVSDUtfUuRXP+vSfH685e9b7/QMH7rIAb4+d/+D1+cvNvEUWphh00G0SnClocbjyadZqrQl8RpQFjklCQtBIM3vh3wrvM8ZmG+d8pv9cJGHbwMXc19yyHJnJDETvQfdCMavKGQZTyvZq358azuZRMGAPsaFW6CnXwdlujWfHj2H07811CdHiBdx3i2jEbaJpm0XJUFxbtaBN37h7TNm4QnW1HbN5lE9xkwgYyWYxWivjsR9+PsFNHOw7wzre/B03Xa/jlz3waL3nNlWh3mE1YZsHPf8HzzsUZZ5ze03NvG2B54ANPgmSvH/sarC5BjZflvOePFLztIPtyw/APTODdMZm9Qtfe2a/pwjj3PId23/g4PvGd7+pExHbckuAzjvLL06ZKRUP1hsaGke8rOnDFJmPzxpka0ZTTRZDRQj/JtI9HinNx5+dnBaHq9GWNPOF4VAI9OSFryvmzLO8yFfIgi82zITQqGNMFYvRc3ADcVLQAOvzXCZpuh75eR5u61Mn/TTUBx6admZ7pNjsYNsSAyyJ6uQimkJrQGQu4oiWjpVLzZbkfV5x/Fs6++BkIkizGJ/bhwx/6FBqMUfJ5vPTi5+Az//YdTdu01JDQc4APf+BqHd7EjmGnx12peSU0hWZgZ6VkUdoJtd/1+/9Ig2yha+o9r/5Auavo3zPHpTeN86aef6/Xq7pxfsjMUgOf/eEPVEsnlEmTT1x5lpMeuLitNjYduQUxazOu24MPRvNMn7V61SqlQdZTl2JgcEAIILVJp11ns1Z3dnwyXkSMWB5w3NVuRvochpix4z1d5G8Rrx18SOaFnbbp/L3O77RN7eff2IGExmSlv6fAVZRhwFZj14vx5ClwKYeCNxZebB4A/y03ALqrorQ8aEXIxsDo8BCe/8wzcfYzztPnXv+5L+G+ex9WF8xJxx+HxflF3PfYE66WwbMA2FxBwb9dNQwDgNxhB85S+yhMrogNopyOqfpEwXoO7rzphympyl00rqeTpjdt6BX8gZvCd4dw0hU1MQjtSBKal0/827cwtchTlFM0eVhRjuYt0YwXYs4Do0PYfMzhOqyI5lY+OZNRNWtsbMxKmSREzMyocEJzPjQ4iGLZXIUQOmnB/1fXm4DXfVbnvmtrS1vS1jxbnk0SOwOQwKEUuKec9gKnvbSXnsDtgdIUCJlnZ3A8xU7ixHYcGw+Z54lACCWkgRAgKVOB3lKmACEOGZx4HiRrnqWtfZ/fu761pdLnKk8e29LW3v////u+NbzrXe9C7stROh91Op7akJ1nLyRufEK/EykURSYVaURXnpFb8TTVo3zNmmCxEzAD7Ispl0zrrC7bkr0UvW7a0UK+IDgmsIbrYx481cLJoVHNigXIaW1stL/7vz5g7/3QX+geb7h+kx3vHlDf28qrr7aHHnzU3jx8xOlgVVXeJVyWsS2bV880Y85C7sTO+aPxa6E9MB0Azn+88LViZUN9iRY1G7HTwiew4D9tgj9e+cK0jYwO2ugINelxEf1cLqzCKusb7Ma77rGRsYIvvAK4aeuht34YgGTalp5xmoIh0Z1SHqqyLHRgTnN5ue19Y4+iZ1JBkDayALILXACBovrsRSzk9PrJ5k/eh0UQ2WIKfzzuQzAEAVeImSq/m8gbs0UXtVlIocYnrKWp2V7ZvVufB/jC6zWpuTTOnM3lAZUC1ERGrhD6Q3iXtYs/+yn78/f/iZ1z3lU2ylBirFxFhc1ra7G//av/0973Fx/Q765ccYMNDY1YRVW53XfHbXbeZVfa0PC4VWRJbSutOldtJ5+yxD591pkl9ywnrTx9RrHbvzczrox/w2FUeZuFr6irNQTw3E/8UZVuloz4fzH/kgKdtqGhfhvo7xHPjxMERCqQhViiaLbveJ89/Mx3bISceBoR43IbGhq1wd4BASInnn6KbxLkT5P6BOkPp5vFZNwZlGA4dt7hWnDWa6qzK3VT/bxCD9JFk7xQwmvUyiWSoSNaIHikaSq2AMeGzm7i2zvxwjti8bGHDx6SLw5M3a2fa8fOPumeGkZ5jFSuYOUVVXbRP37CPvahP7OxiTErL5bbhZessr7hwVJ9YF5Ls33yzI/a6e97l+bW3rr5DkG5bXPabOXyK+zK1dfZ1DT0NLIbh68/9ekzbemyJQmjjyFFDmyJZJkImRGTKRZTvJEKPL/8wVPFLHZfKdLMFzcwG579r7Ges1X7+o7bYH+fHkplzjFx57MnHRp2fzZjX//Bv9mLr79pY1PTIhYAWHQf6xad6MTTTlYO63VkR76Ae0XWmPaBQSwmChQUPKj4IaoEDWtyKs1uhWyQkCtRq9Vc4eVZOPgEU4Jkqd2X/LMDO0Q+QtuS/JlX2aZtoLfX5+6Me8SuOCBlDWqc1Ewel0VNp0YPlrEs+N6Vl11s/8cZp2mEKcdb6Np0mV142TXWOzis3ye1nN/eah//xF/bO05/p3372y/Yt771gjbF5ZddKM7ffQ89rnurylVZZXpOGzauKrVuz14b71FMGH6pVO3Bu+TZo9bw6399ugi6U54oxrFDSsWXPwJrwnxwUnqPd1tvbxf9jG7yknBh7K5Ib8SRs6Ld9rVvWtfggE1OeH38eNdxGx0ascVLT7BslUt0ccpFhkgsGnrU5CpFnypo2iVpFyYPd1JV7SPNggZFCkX0r0pdRc5pT4gsTnoBRpG5pmI6HKsKmrphnLbE7/Ue7ylV8XwGruvc6jDHeLGEoP2xKW1rqLV7d+2Q8jUz4tHpY2hh7A0sziWXr7KB4RFt3urKSmtvbbKPf/yjtuzUU2zTplutu3tAz2DjxnX2nef+xb79wve9M9bKpAmAZbxhw7ViA8emi8XWus2ur6TFn12QUVT/mx8/W8RsVtbVKZUKzvz/38ILiJiatKPHDtrxrmMOqGRhq4xbQ0OdR76iKGdUYXLyAtQp2LRlduODjwsRm6bXbmJK7wG/bu7bFjijNlPmkxdzHs0L8k1Yusw2hY8xoN5Kfb+6psZPU6RsjAdPzRK4GRZN8irqn/NNhO93yNZzfRDCgwcPeaahnzlHLZqrQwtIFbIUs0mnz/XX5RLmtLfZI7t2WFkmFW2o7lERTGij3KgqekW7YvkK6x+gszhj+YpKa21ttE984n/Zyacus3XrblR9o6q6zG7eeKNtu/V2e/XNvUpr2bCtrc1WXpGxdetXKo2L9Yrhi1E/iawrFrw0MQPYmcD3Nz95tshfsvnqmVGUs4oAsxUewhocPLDXBgd7rRZeO4CLUgLUJp3gr6JBSnV4qAzrpazJDp/IVtj6ux+08XEXIOrp6rburi72bhpGAAAgAElEQVQ75R2nWi5fJVpWTIuWdEcmK5WpoBITsU6NjothorKsumYq1FnDahJjSAOHiD0hhsQhWqRUL1eRZXLCTl12sv3+dy/p+zBo8dke3KWWyoT5RwnWT1XS403ZwalvW2wb1q6yGvAHZt8orYJXMCZ9v/8SBxeKduXVq6y/f0TpcS6btY62Vvvfn/yELT5hia1be4Ng7o//Px+z//7f/9SuX7fZDnV1C/cA76+rr7X/9t9Ot7/+m//pZUNflFKNI1SqWWjJzKT0TsLb9CUmjoIWXpEqIkJqNPgjiYlQdhbiNWl73nzd8hUAAVM6QbW1TIScLFXUWCzMLQ8eU6uHKdpUQWaNhzc2VbRVdz8iXzvQP2DDA4MKZIBvS0UWsPKJcUX2oH20PQnmRA8Gf54ia95P/w5lZvXDe4Qr3ZuE2omQmS3X3Ly+48fVri3oGWsSfjHQykRsEOkyNWzoz1Te5Tc+eebH7NOf+JiVic8fEqN+qpW3o10z2F9iNpWCQCvaimuusy4NcCK9q7B58+fY587+jO154y372teeUoFn545bRL9esXK9DQyOKACtq6nS2Jfzzj/b5syZ4zUTLdfMBogTrhOffhLiNbGh9TMWXgUH8B3pw/6RyH+KfNlBv3/pRWtpbVSwg4hIZUWVFgUkiTcLnhxBhEqjqp5VauFFa05pVKE4YdduvNsK9XWS7oSQSLfI0tNOSRRh5qP5o4oqXq7CdXNQfFQzQUrB4kaD9IirCN9NLd+LKR5TkB3wRZzgNKqssgmdBsq0iaemVm91nrjlkD0rFq2hps5uXLfWTjnxBCtOjNjE6JBNF9OoD6EiaeEpKKmBdEjmPsy8HnwmY2vW3mgHDxyVqa+qyFnHnFY755yz7Stf+arteeNNETm33rpBa3HJZVfbRKGo3L+utloLf926Vcm3J1WwpK9TMu+zOIhR7ZRf5z+58wzI3bNF/Bw0qap8zQwpD3CCFl8gycKk/fxnP7Y6nW5Mablm0kRtOJgutAHzoNVpGukDTQnw4NOAez3MwqRduXqrldXUWqEmp46b0aFRW3jCPB/Gm6pPXjIlGnWFKZogRGAYGxcaqNl3IVGCWeUI0cQwNq7UjxPeP9Dv7ohWbIE1nutrkzKIIE3OUPqTpETGoSinqdMANR9835/amiuvtPKi2ah634gbmLfjA5SC2RMBltDHXKWNDg1IRzdcJDgF6eimzV+wPa/vLZWYO+e027nnnmO7du6yvoERe9/732Wf+ew/2NDAiF199RoJOWBl6eVrbKy19etWWyEdDA9WnV41m41DZ66upyQL7ylfVCW18DwsdGkrq/PqWg2TwALRqPevP3zB5s1p18PioSslKjI9sqYEYPBv0LMQHyZ6la4MHHSkRRPY4cWNgl25ZqsNDY7ZZFJT/qu//JDt3vOGjQGkZKkbx8hxCi4geUNC0UT2EE3Z+XlAoZxexpqqmRLqUlKB4JRE+TR2vrc3BZ07DQtOOS9WT8BMgXbirJ115sftr//yz60yBAJxIakEy3Pxh+sNlVrcVOjigQPYTIwjYDaDi0RN5LZd99qvf/Vb/QYWcV7nHDv/gvNs88bNNjw2affct0uiDj/50U/t4UeeUNBLCkxgh4u9Yf0am549blWAES4v9QSIfTNLVj3a2tN8HFkGsHr+AnyKOSwkCQlFvoUJ+97zz9mC+XNLrUPUkTkdBG38Hg/K25jSlIbkU928uYq0s2UyOoFu7op2+bWbbHQUwWL3ids3X2vNjY32Vtcxu/OpbynIms4SKnncgUw65n1oYKjkNnhw1No5wQgmkwpiobzWjXIkMLzntJ4ZzPhgXTPbSySGgk1PeD0cw/+h95xhl1580cwpUtk+gTZJf4aYQSdM/p0W7TQYSBOoIVKaDfb3ei1cQaHzCCnFPvTQl+0nP/2Zfrc6l7M5nW32sb/9qN1//6M2VZi0u+7eqef58EOP249/8gvLVVWoXeqEE5fYqacttb/6q494FlOqqDocoRi7VF53/19q2UoFptikmV/99FktfCg1lFUjLwKJYdx+8MIL9rYl80oX7sAIxREP1hzzpuqWFpRJjZU0BjjJMVIfZ8b61CQPmKbsipWbbWh4TH6Mn9+983qr1M8mbaJQbhseecSmilkrpJ1LkYeawMjQqDN3ktwqAaLy81SM8I5ZFzwQ8yY0bpPbIOAsFZhgoKZIHez702eeaZ/827+xbMYBHW3eWXNrg7vnTYre8oQLCVPuuZUTPMrLM5rS4dCtT5f2RSmzJ77ydXv+hR/q3/nKKmtorLWLLj7brr9hs7W3t9qKa5dbTU2t7dh+u/3htf0im1SUZWzBwnl24UXnys/roCVwYAY2jgifR12wF1980d71rneVXIBboqQfHAuPaNAogVoNufekff/57+gimhpqZ/htSXXaETAvd0bO7IvvBZAwO5xULyrgGjwAVTm0vNwuu+Ym0Ydj4W/ftlYkTtiuba2tiop3fPmf7EAv4gRaAu3eqfEp61HBxrn0sF2EUSeeuQKxSCeT4qNOoEy8/8y7TxBKKLdcJmNn/93H7S//x59bVZXz54Xvp8jeEb0Z90c2EbFCtGPF5lIRKfUE4ttHhocS3Suwe8fSv/P8D+3Jrz5dGsXe3tZqly0/Rw0mdO+wyeEu7Npxjx093qvnVYuSRUOtrb3u2pIiJsGoW9YY5SJH6qQP/kucwzj1EeknU/+sOmlYNAYHEUA9/fRTdvLJJ+qGCXLYcW6yEidb0bJDnDxQmbBZYzuFf6dxozHvPRZDQVW2wi5cfr0NDbvCJH7ujm3rhANUotGiuyGarrSf/eFl+9Lz38O5+jUUnWHTfeyYn6BUD4/F8YDQF1dky5ioHLku+IKZzW9pspvWrLD2+nrvLk26PCI6pA5dPcA0GCk2gOP4bvaDCqZzLDVtmh99mANZiluWJJU+i7j6rz/9ud13/yMKRCGcNNbX2YpVl1p1dXQQZ8VfuG7NRhseG9ZmbKqrs6rqClu95pq0FgCSKY1TQhGMx1my6SVqmd8Hr9GhpUnzVz/9pky92o6GR+0H33vBFi5aIOozJru+Nu+88SLFjBk834WC3SRi1nkgihjl99ko3sHhgVROKZiozsCvmaxdsXJTCthM379n140qENH/Hu9DuZQHN5HJ2LV33O8AROo2IVXr6+3zjtxEeIgALiJcFt55Zj6bDbPN6Xpww3orKxu3wnSZGD+FIqVTb2TgofC8iBf4S2QE/AnCCWLnnD6PH/izpImfNOZgzzJwwQcl+eKE/Dob9Pe799jNm7eKOs4haG5usFWrL1fU7uaYg2V21fLrQEv0LNubm62uIW9nn/0PrgyKi0nxS3AHFUeAxaSNHHN3JLUOd5/ANU3+yPzyJ98octqBQr/1jaftnW8/Tdx1ghcWlO+HooKCiRTQOfFgZgge9fN5nXOVdsUpd7NeUSJMRmcKC3Xt2lu18Fw8alcP3rlRHHTyScAKoU78fuqfw7Uc7h22TffdZ4VMJbwTmxgfs5HjA15jV+UpzVwTugbxg66TolVDy8rmbH5tld26eb3oymEVwjopABRVimmODkBxjqJZg00nV5WYupoNk1IltzJZUchp1BSSmBpK/1OKpdebdR/rtWvW3KgaAYgc+fkN66+xyrx3DWsDT2ftokuvVhNmLpe1zvZWe/s7ltlf/MWf6RoEa6eqYty74whpzFnqsIkMzWv0qbmCLODn//rPRdifzz33rC07cYnVVNFYjyKEY+Z6gCB7oi27VruQqfSQ9drU5kSlie+7frw//JK/LRSsurrGwZVCwVasuUUiAgA1oH93blsnwqWbZg+c5NNTuTWTqbCqykSxKmZscHTSrrt5i40VfIePFt0X47OrMlmbP7fT1lxxvvD3J/7pafvO935gnS0tduut14t4ETlt+HK5nOq8TjUBGqdYFLCkJOHjv5JJTaFxIHv6fHoBFAzGwMQU1AmrD1DMad0T41N24WUrFOzyzBoaau2mDSstW5Hg4qLZm2/ut1u27rKKcsx/xpYsmGvLr7rEMpmC1iWYxbMnRUe6GJM9ZMmTJaahItyhNuxPn3+8+N3vvmCnnbo0MTxc4iNStWC3KlKW6pQL7Qgpc/6+m0janBOYQt+7QI00CpTXw58bEUyK6obZVWtvsf6BARVramvydt8dN2vufHkGnRifkEzs4PPnvDrn4zNnePQrV9xcaoxQWiWt16w1NtZZ59x2u+DCz+l7Tz3zHXvyqW/a/JZ6u+ULG8UbCHMoM5w2gqJvYbyJmyC1rcSizbqbixgioiosgtqjmQ+LsGAqAPlrneipDt00akVoopXZ2ede5oTMigprqK22LRuvs0yFxyZsqPvvfcx+8eJLum9g3faOZlu9ZoW08pIivehlIe8+E8DGjJ/AFhJHIG3agLgzG1aeXWxrb5NClSSzcg5IBMghdAzfLUDGNdD53ynGng55O5J3YuLPKQQoDYLsQJ1elkOgsDdNTE/blas3W08veDX4ed7u2L5edfuKLPECVsSDLKjOcdpwG8C/nmZlbPW1G0Wj1olSX7gLLpRnM7bkhAX2+c//g0zwd773Y3v4sSdtYWujrb95re41uGhebk3zWCPVic2VzL3nhCYNHv6OSS8FkOL50biAOINvmBIXY1ZziJtc6U1bMVNuZ597qTpmWNimurxt3XKDwciLrGjjTVtt3yFK3rRHl6mCt/a6lYp5mPghYCqGKSWmUaSVgqFnz6FN4JIsgdZryjIP3bamKJECpj4nJQf0UllwuO1cMN9n8UhznNPuu4jXxIWGuY/GhdmuwLMGtxLezZq1q1Zvse6efvW7N9fX2q6dN8qiUL/WZ03RxeradVLByniaKECoSGlx1G6+eZf14S6IVBWJ5xQYMQh44aK59pnPfkp0rkNHj9rv//CGnXbyMlu0uFN0anrl8MVsJty2UjivcWrhnPvuZVUWLJfzThgBPtqYbr4DyOHa3D07WBVBb4xOdTTZlbimy8rt3PMut1GqotmsNdbl7datN6q8LZ6AmV276iYbHByWBauryduczla78qpLne8fbVJp4UMggusrtYZhOXhuCUAS6kmwGdnFU49uKfJwpJScfGz4AoEwqTpFJEmRI3xiFEViZ4m6m7a6pLaS6A+vj4fA+7LBeGRXrtxkXT39+vu8jlbbtPFa3xjlDiCRiaoZMgkjwWzJV6NQ6WkJVmPj5tutq+t4+r0Ka2ioFyO1sanOOjpa7JOfOlNmloCLY4I1IXLOZXMCmlLeWLIirpU341pYBLF1vX6XXh8m3Is30eEzG0SLDRB6dv4MQ8QYQnTWLrz4KhtJHT51+UrbsWOTwKuQTrl6xY02xgiVsqzV19baR/7nn9uHPvxBT1Ol7emB9ezgkc/l50o92ZRcO+4mYfmy1jFo6smHNxWJ3Gvzdd6tAsslpSu6UwV6iOL693kQ0XzAQkTBgw8jOnfzk1QhJj3FC2mxMEGUVq9dt8WOdPWqy2XJwg5bv+Yq158LkaCCYwFkCyx+c2tLqWMmINC77njE9uzZ50ui4MXZMvnqnL3thIX2d5/8XzpR6MjA2OEhEUVzeh2EcuuFC/NbTQydNILUv+dMW9+MiC0kD6vx5kkpOymGJ6hA7ztTxp0hiWCqBABZwS6/Yr1TyOAVVOZs584bS5ItLOoFF6+wTJlr9rQ21tt1668pSbUQJM1G61iTCLi5ZpWpIYKAaqaRrtRdWAusreKsrzy0qYhpAjiRZKeK9y4XonRMunBJICDVvLEQ6lWnUpceXpjxvr4+q63NJ/66CRCKFEUdKdPTlq+qtKvXbLajiCRZxk5/x1LbeMNqO9blFGJF3DKvvjC4ABSZS+yeJIT81a88a7/4+a89709SnpA9GmvzMvX/++99DjubmSAM8851VlfVyE3lESdOSKMTKWPIQFK5VueJ067ollUDBUp1Sh+9UMXChPXDlJcoVknXPho6FOJp6GLGJqen7LLL19nwiAsmsJluv32jmEK8fnh4zK5ZeaO6Xri+jpZmW37VBdbYWJ+yJdq93QLp2SSOXUi6qlsoiUXF4k9Oem2hIFZQ0TLPPLHTYf3EEC09iFS/hdzoJ9bLmhL2Gxv3CY4CRvyUicqcfocLUJBFPp6CDPHjk3+hpLnu5tusq3vArDhuH/nIB+3sf/h76bROTjnOz0KJbDmbNJneV71ykwX70Q//zb713A9SC5F5kakwaTVVNbZkcYedfe5ZJb8dUzV0ipl7kNqQfAqVjLPex/vrPHMQbSyJL+kBaayIl6rDWkARE7CUBhGT+noeP0Nr1sZELpyYARZxttwuv+I6G8CHp8aQ23deL3CKNHLfgWO2+dbbdVX8bltrk61bd40GNrAxSB1j7h4Qt0u4eWVR1PJZqXb4eFwkhJviNHqAE5b55y/vKEpdKqlO8QbSR2WokJoVsq7QkM+rqUDyImmjBEZNYKWO0tR2hAsI9E3pA/1psQkSiLFq3a12+FiflZcV7NzzPmMf/NM/MXYlpd1SO1OKntX/HsP1Un9aVWXefvbvv7SvPPmML1sCLthnNZV5W7yo3c694LM2gFxYdbV67Fx0AMq2F410f0HhKqlJO3PWeXze9qTYJQ0+ZuEduHLLhDXxTCe1Zycp2IgVPNjDiqYp2slDL79yvQJTMY4yGXv04S/YxCgzP8yefe5f7BvPfV/3xeZfvGiBnXvO3wvoYWGVVeF6RVObae2KjVLadLq+mfmBauWachmXzDNP7tJ9STSf+6P5AHpUak3izSXMM6szQ3LiibvNRXDS/cykScVRjEmSXlgETqmiYtKJyQnbcMtdduhIt0zW+uuusCXz5uk9AJMUF9Q4kBTyJ3yPVqXmlhaJKtRW5+3F37xsDz/6pCYS4YmVhmbM8tWVtnjRXDv/ws9pEfF3LDqxjNIwtRNFFO4+XlIkImqSK3ljI6cJV0Yc4q1UTufyeAewKXHVWeyyjDZXTY2TUBzV45ky9mw2G9aVsq66+gY7drxHz5Hq0UP3bnFpNdi1W3bZwf2HBSXn8zn7m49+2P7sgx/QhA8xmypcFSwieFqp9T4zd1WCk9lwMUJFC53EETL//JVdRS+0ZA3/jE9nN4cEiSDNFO0TaHHyWTy1IScqNLtesqOSFnXmZwnqTREP5ghUTOlexuy6m3bZocNdetB33r7ZMgValLPSveXhYvKxHIj3ElOw87kWsgvy6FxFue3dd8juuONhMVcjd6anLJ+vtPlz2+wfP/spvScPRi3XqeUZEMjTTp9Dq02dsIMo7tCdwzw4ZStpfrteA0aRhvTOLnzAk/PBQNTlgZvDgzoJNMxvIgnZqlUbNe81AuqH7tta6nK94sr1nl4WM1ZTW2nXrb7GqvMMJUjCy5p26WNbWUzkY4LVzLrwjAKMinm6cnFYsDQFK/PNf7pLZd3x0RHh7J0dc7SoAcWyMCxqgPwK4ngoY+jI5RxXTjVn2C+8nofKe0SKp0i7psb6epHppJW5zDZsucv27ieYm7Z7d22x0VHXguVzaY863tWtMnFbe6tj0gUX7yNvlpVJzYq3bnvEo/FS9cuspjpnC+Z22OfPPat0+jhJdOnILKv44+6BgI2TpDRITSGkfIg4OOvWT6+3OuHyAgQhaJVaRsbUYRvQKe8fVObIhlIQUar9Y1k23LTd9h44oh9hrR6+f5sXfjIZu+SS1Z6wZZBmr7atW9bLGmDXBBOnnr3gAgwMuhvz4pLrB0iBi6JNqilEql1iCX376/cWCWIYBshDr6eBsqxMZkunOBEWuUBSIXwtUOv8BfPVBaN8PeXamobADhwaKvlOHrgmH/NwKirE3CG6WnfzLtu3H8Jh0e697RYbGOwRT46NEf1uLmrkSo35KsfxNWAHiLSsTDoyW7c/Unp4oZbFaxfOa7eLLz1P2EOASogQuniiq2ViNuvqanXvwdlHWw8zEOLE9Oi3d3R446OkQV0xm9erkjcrBhD1WzJrnh56U8esQFFyJCCgGbvzrkft57/6rbue4rRx4r3nLmMXXrhSXAGRMatz9oVbb/BYIJl0hiV7FuLWhdgLy8VnKT7JmA3098t60mAZBaUA0aTg8fSXdxRJCWCv8tBZIE5+Hb3n2awWW8EWQgac9sqcbhqzjWaqWogSpTp2VcmspGmVIUYUYANuZMuO++2NvfsE2Ny49nKrqnJFDCL+uXPnWm9vt/h9mHuiUTBqmgoamMhUkbPjfT3Syt207eFSJOtgDx0nRevsbLeLL/mcyq0jzMqh0saJ1agSBBRzSblaOtNKrSR/htCR3FZE9TktOm3bbAoWU0JNqUGzVPhI9GtMKbUGzC/uM0rWOqmSP4XoMWZfeuIb9qOf/ruXbqen7aEHtrklmyjapcvXlizVkiVzbMVVl800iRDHJFfiwxbR05mWRWVD8qxiQ7ju3ozsCwuuRhA+876dq4twzcnvhoaGdcNNzc06ZWwAgistSNJiV2SMhPew5/IaQq+pkS4jovp1ivypPGGuBQer6lXU6afosGn73bb3wCGhads2rrL6hjrr7e21fGVOFqOmNq9AL4KRfB5LwAiQvC8SsmeZrF2/8Z6S7lygisQQcNXPOedT/6mowoNtaW627u4ebQQWX0UgJMxSB02oWChQUq48Q1dSeprN6p7AFbAexD3yqakti4VXL37aOPLvCXbmT8Ajspenn/kXe/bbz/v7F6bt/vu2CBc43jVoN2zc7nX5TMbOOutMe/97353qFR6QBtaRiEkJeaSJM5uGFVBPcJcY/IzI+wPFyzz12Db9fn9vr8y6JjAg3znOhMcaO9bVJRlSpQCa4JzznF18cadWCRiQP0Hsl8DLBXOl9ZYqfT7IB7/j+ey22x+w/QeOyjzt2LTWxidHxbEnIg+aFO+Zr8qnaNwnV/GAWbDJKd/dW3Y85sIJjhK577aiLVzQaeedd1YJU/fqmJ8WeAEekfsQhND04b5C3YprwISWxpmkBRQ5RYOKvFAliXBhDQm/T/AoboUrIThlc7Q2Nycl7kptjH/53r/Z40885fWfqWm7686bREP/2X/81h770lNpgTN2w/oV1tpSn4gkXq8I0Cj8tQLKcDnJCmhRU2XQM4yUgUiZI2OZB3etLerBpeCovb1dN0KgI5Rpako36qXHENrznBRhQt6UBSDCZcE1hVGRI6ifpxj45SjiuBLkuH35q8/Y7lf32vve/z778J+9x6oqMtZY16AuU8zf8PCAhuqRaYj1guhPmhwtl0JaODFht+583KN1wff+8Cn0zJvbYuee849Q9EvmNkgkWB+v4nl/XnXeCzDE6ywms2DYqPj56LSJdEnVskSAkB+PPJ6MRhp7KHcXrLbOhxPFEEDh/lOTcplcx+4/7LG77nncpssgik7bPbdvsInRcXvya9+2X/92t1c1c1m7bftNNlmYSDAwFctE7kzgTqCGKhKBpSRsIhBV35z+O5HWsUkyD912XRHzLT+O8lQFPnFE9XNyeRoAJEeKxnxlpcuGxulJ/eE8DFA9ImF0aWQFCtOucjHpUqUsDnGBFC6nRq2vf8TaOxdY30CftTfVCFQhnqDsSO86Pp8ty4WrgVEzU53gqdoCM2anp+yW7V/0DpkUvbLwbLh5c1vtwgvOFo8vGLNcC58fU5s0OEnux+VRsVDcBxMmws9z35SbOT16JggQp4kVGvaX5MSoafDePAusppetedppmEHiDDJlA637w0d6bOftD9oU7RKT03b7jvVS6F69dpONT7lJrygv2vatN6R+f2/R5n0JgiNeioYJXi8cgdgs2Eiix3n9QdZ4zGf/lhY+UjcJC6RZK/yd00+jfnDleEgENvh+HiILSbDFG9bV15dwb3xgCPFhmicm0wAclXLZOFM2MubBGgFJU3OTTU2OiWpMoSYw+YgHuCmkTzipOvkEZpzOyQnbftvjdrynr+QTxQ0sy9rCBR12ySXnCgZmU3M/nFriEs19b2jQQ+F/dbjU1np9IbFWgEVZaH4Gd48NpbI0zBxqGmk2nvDxVP8Omhgug0AQcYM4iQR86v2bnNR99A0M2+atd4uUQaq665bVet+r19wiS8RXS0utrVtzpahXDh+7mw12b4A4ZCkREwQaCVfC3WKlN7Jq5NqsqdrPffUOVec4NQFfhnnG1LHzAUwI+PhApSipVs3rWfyYDs2Hs+gsGD8bGurTQ6mqIlAb14Ai3gPW7vAI05XGRSnm9zEenDhOPBRlqURD5EReTGM33GSz8SR4hFTY+Jjd++DX7fCRLl+wZOoJ+uZ2ttglF39eboVNiG4OqRnRb2AToYQp7kDykTz8GDEWuTndujR8Ks+vdNWNqJtjXsPPqwyaKnnyqXQRkTqlmrhKpQwsmJy0o929tnX7/TYOUlqctju2rpE41OobvpCGIJudddbH7U//5FTxECOg00ZKuLzirtR6Hd8PX88aB4jm2ZZDz7FBMvfvWF3kwXsfe4UEh/bu3VuqrXNC+CgX7Eecr0IkR+XmExMym1oYhuPy2oxDl/y7KhUrOHWcMjVCVFRYXUOj97mn2vHSk06yPa+9qt1Zm3dql5vgKQESwqaTADEwRvTb4wLuuvdLtnf/4cBIPPjJZmxOe6tdcP5nk0q1qzlSl48TyGIp2k4Vx4CTQ1YV7r6gaYIEPThXsI7R4qBqLL4zV71FWhi+mLVeB/DeA7cibOYgdvT199r4ZNHWb75H/Yll0wXbvmmVmiCu23CHW5NCwbZsWmkNDXnXmJ+loKl4JPl6ucLUnuYTrD2IizQzYgBxJmdRvDNPPri5qFku5eVKdfBv+HR8ReSyfIh058fGramxUZOeQwUa0p/06Kp9Hhw3J6nS2tpSJwkVM77UKl1drWIOvppNIOVo2rAy5s2WVJGkLJkGBwFiJFCH08r4Ut/97p+/+8L/az/6yb8nUoSbMtK5OR2ttnrVlUltclJsov6BvpIrkwImLqC83A4dPmxnnNp7wtEAACAASURBVHGG7d+/P20cFzyk946v0RGkWP1gEHuoOFNI/HQtEtVIL/mCZsIeHh52EAslbmfwuGz5wADACmXhCVt5/Q4bROuvttZWX3WehgJuuOU+cRd57Y5ta62y0q2Gl3T91AaHD0EJAl9POJ14QeMr68kaIBUzu1gWLl2bgRMvOHNyUmkbAR1ADr6NXYOf53TqgZaViTwQ/5bWfEKmODm8BwEOE3m8uodvn3bwowbhYpSsahXxk+ZJ7EjtVhU2PTGu08PvifWik+vTJAI0UmtSBbDujMn68b/92p57/kczJAaB4UXraGu2Sy75vD7PpUhclQq0TeBTZaUNj7hvx2+KXZvJqO88AlG+R8Ap8inFGXwmQ4/QpZ10N8hmlYpXb59iFhhZfhp9ALCSTJlnL37JGihtnLDBgSERSYDAW1oarLd/xB59/DkFfOUZAr4NUr8oSxp7bDanpSW9H03PxAV54ciD7jRRUi7HSTQ6uMz7FZTr5eLMfdtXleRRiBbZaSw8lTAwc0w/1TAV+4FjBweFZXMDkiVFA25iwos2lZVqbyIXl79XLd/noHkg4mpSfuK9i4SNxe4c6utRkIf16Dp2TA+VGKMhjSP3ua/MdEWe2xEoLPBrew7ZV772zRmdPh500ayjvcWuXH6BTtro6LATRhIW7s0gBUXz3G/QpOMABOIWFoyUTGmZ6tmetlIdYFOxpG45/MTTg8c3WVjPnRl4QDXPMx9VNUPjvrzcjh3rsjGJPUyoU+bbz/+HvfTSK/aRD73f3v3OU0QjYw1k/pNiFfcUMKxKsEm2XDSwtLDMo5UGf5KlgTIewZ024z3brlV1TunMLMIgb6CHklgoBDTHjh3TYvE/pp5Ai0XjxLCz0GZXBC1JFMAPj045FZ6XVgl1Q+mivqFBwAbvAZefzhOsA12vnqZHH56f+Gw5phKs3LONnj4Yuhl75fU99qXHv1k6WREftLe32PLLztECtLd1iIeeS+NJXRfeewTpVcM/e7nWI2fSWSwULof75+HREsU4NJ4JQR6bxxnIfqLk+niPSUaCIVPuvQUQKLkmCUgkBlBg5vw+vQVo93FwYNmyOZmRg0VkA7uCd073jJXSGqVpWQHKDDN5S82sHrkHTyAkVbFkfb390jQQykpQeN8XVhYx35yuzrlzZWZZdD6YD+MEYqoxf0TGXCw3HmYrAhHMF5EvEiOcJAKjU0492d58881SH93AgOf1gXpFqzVtUJXykc6yZUEEqkwVrLW1xWe0ChFz009f/sDQoBb7SHePPfjAP5U2bUT3bW3NdulFn1WRgnQHISbwcyhU1Arw+ceOHUkyKv4wdBKS+dRg4YTK8Z6cZMQQCSxZUdI9CjwgvnJxQ0OOeoIjqObgVCf+HXT1oHFFNsFocg5DSTE8658xMjik9+BZzu3stOPHfXgTh0ULCzO5qVkHyOH0mVZtguFjR49plDmvDT4DUARunH/LJRDccWGcxDid8m1J/owXeTQ641cJHjgZHrABsLgfA3L1TkbHwStSmRUxA7B9Bg9wOggOxfhJKhli8PYOyL3gJubPX2D79r2pDbZg/nxh+MyKdxi5rtRdg9sYGR23W7c9YNAdImJnYdpbWuyiiz5tSKgA7iDAFOihIngsVlVOkKoIGIksIi4BSGZCwaSsmUrN+M8RMpqEjjk66vKnWBB6+FlUucBJ9HtqJYIk0Qj6DhNFjSd0YP8+65jToc0caJuzoMo0WkxoZOpNJMbk2rE+nOLWlhbda1hp0kDoYiIfS7K0zMYmvVTMQivwm0hzcxltysF94el7JXdGHo854oHwIVwEJx3zQIAjCDeZsxICVlvrKRraqtTgB4c89ROdyCxXRdsvc9Rm0g8eIgUZ3pub6JzbaYcPHxblGdmSpoZ6uQAsgEaI5SpcqjQ1OdCGFZuQGxoZG7ONm+8RgdHXwQmN7a2ttuLq88TH91nvHpNgTQBWlixZbAf27XV+HTBKmoAVhSQ2PPfOtej+E2DlwxfGSj0Hk+PumvDjoHYcCLlITYigquh+nWMp/AN6mmhkMSTIRBQR2AKqpgDQZ9UyVNC5fd74qSJPYvByaDra2/UssjR8pp5G75fM2uDIoAJ0GEu8J8yg8P8K7p56dGuR3Xrw4EEFVbX5Gk89in7jbAahXgzOZUGSXjy5Ovw4bi4qeMh0RXTP08BN6LSOky56kMNO5f3EdFFXicmcHT18RClQfW2dNOr5u/rFxz0VjNSPhyrAKIk0DY2O2LYvPCwlTPl350xaW3OjXXLp5xL0C7fcIV83s2U66SCF1dV5BYq4MaJ8KWwB4mBdamt9DnwaJYaPnanJ039OwJeIIeOjOvW8P/eIi+G1ZAFh2hXYJa4cr+FeuGZ+TvosskearsWfHEYWaWCwX+VpuI3CM1IbN88QYE15PYcSVDFN04TQGV1OakIt82oi5FAJPN+86vNFOmcOHTzo82KYA0NAQ15NLp9oVujEUzBhARSoaMqykxV5oF7R86Apeu/YYa5ekZFPOnrsiCJUvtfb22Mtra1aALIJ/BI3m2d6hUZhT1hn51zrp6M2je12IMSHApHH8/6UZ9ffsMuZp5hCFSMKWvgVKy5W0aeqslqdfDKfAmO85RndOFJMABBNhEIFKxVgSgBIykBYRH4XtxTxgIK0NJYb2RPuq4Q5CIhCQNEbNORXVW+fKEHEXIkvSnD1/f5kuczJFHKnBReVAtlUgJjyMKXS4hk6stfY3KTAT2BRUvEkm2FThJoZ8ZU4AET1BDKB3ukkFoulQobSq64ulWgx2dJwTaO6XfKjwnJV1TJN1My5cTYIX5HqiVLMOPGmJlmI+JnAG7FyauzwYachQcLg88gI2CREvexyfhfaFXPaBSyl5kJYpFu/8ID0dOS7U8Nlc1O9rVp5hbRfVTYuEJn7MILpwqQCJzIJAKnxca9gaQa96vAuPe4pqVfyWHhlJpWVCb93AcV8jc/VQ+SRe4Eyxu91dnbIiioDSkicov3ETYiN5fyGGfkYZQjQvVKgyXNVYSilnd6945E7VoKNxJcXrmpLimOIWJGFsFayPFUuRhl9jZk7brlKvXOc4qVLl9qBAwf0oMLH4X+5ccyc+wrGfo4IPaJCJohUzQZAlFnNQeUC2MWcgCA6AA719/dpNxK88OVRuqNOXKBvnhrr7JxjXV3H3IRly23JkiXCErhZFonNyBefic/dvOUeG5GQkpyH3qupqd7Wrr7SpqbG1aXLPSxatFjz7tiIPgfOu02HBgls/RipxQsRzHRCuTpew73weQ445YTq4fqQceX7lRWeQxPn8Bp8O6cZ9IyDwCbms0WuTPPwuKbgJuo5UuwhSE7TtLQOafCwIOxU4FETaUqT+VMVRBXDnOrFe9U3Nsq18vmaZJ3z554HUcUdPbBzjRQxyLV5QVSywgfVCfmCkzeskRqqX1d72bWxqVFMj4qqKkGRLc0tQvZiDCe4tZdEvcGClIyM4KSlJ9rhQ4dV8QIQUt2aGfSCdGlxctIlG6Cnpzfx5MgGhtEjVhwRp3B0ZMx23v6Q9Q8RiYsCJ1OPysT2bTeL0/fWWwRxXtIFTSTadnSNBgrH1MmDfeNxj6N6+N6gUVBXb6RGkQcPDwwoiub1vA4iJCDT5Dg8QUfHQjc/3AfPhoWJqppQP4KytBmi2zbiBJ4dC8e/OZgKvtM4E0G4QuSmZCUJ5KIoo98vK7P58+cp8GSj5MBfqiqtd2DA0+aHdq1V349gypERW7xkiXYoH8omqKmu1oPioXd0tCvoIjjgZKjzVcN33Q8TQfN9plRwwVTj8OXKy1nQqry+DyCxZ88emWzmx0RDJic5YFz3847wMYMWc8rNNja3lJo3dfNl5bZ9xwN2uKvXyQoSMTQt/FXLL1B2wIZgOLBSoFT544EQvPo0rH4bGhoUYKLMJevSIdFBrJsjJUq8BKGOlRVyFzx8Veum3NVMjsFBdHcZiCDP8Y9TSd7P9fm8cYUTC/dBAdnUlDaUroHa+6zysdLrRF5l4/D5mH5QVoLzUO5g4XHPXJMscHlWaOgodDYi/3u3XVsEg8YUs2vmz5tnBw4c9FNAwMaAPem1wsVjisSw+1EK/0PEBjXin/NQTznlND0g1J727d9X0ogFHQPpqqqu0ebp6u4qQbPQmzw4rJArwG9pU6UCDuYKCyAs3YpWla8tVZ686FBhd979mO0/1OWroxJrRgu//PLzFXfwu+IMjk/IauH7sFyaDZOrUPZARTIfRJM02I+NxP+AM2wIOAccCj3MfLVP1NB0aDKAvHrfNB9+2qN1FW1SSsufvJ50j4yIwJb3xcosXLhQCKiyIyZWzJ0rF8DPgvdIhM+z4ftYBtaM9+HeOHykbaScvBfumc+m7q9CESqflWzwPuvonOPj2+/ccrWoV1wYaBbzVkgdADHYfZwI9a2rQW/Cautq7Pjxbgcp1EAxba3tbfqgBQsWKdh4Y88eFTuOHDooszw27sI7oF7sUuriUaliUZubW3SiOflAsTwAuO64noiS+Tz52dS3xg25WZ60+x940vbsO5gWHuyaIQaNdv26a7QoAEbsekAkHzgMT5CT4DFKvrbaDhw8YFUpwuZ7nDYHZWDo+hcnU6kX7WRj4x58DvQpI8iD4jHQgGKMmlK8hZnTzmcr4E0NmNQ6cA9YPT6H585z4b6BxTnFfAbIHlYp6FZ8NoeR9YELGVQyFj6wF/7OBuN5UW3kT/7NpuU91QcJzsLCk7bh8BU9TkyKY0dAwwvZUUqAKP8Jqhy1uroal+lqblVRprwypwAMTdr9Bw4odyf9Q/bTOZBOoYrgiL9zs9w0sDCvJwBbtHCRHTh8SNaAYKmXacpJDIFNwyaorW9Q1B9AEzoCTz/zPfvliy95mqfGTZMcyoqrL07TrEflQg4c2K8HXFvr0Ce+kWvp7nUixwAQKrl6UgHhZHGSCHjD9NfXU2MYkHii/Pi0y6SjOQdbloVXrp1m6bCQPF/undezCByCUPrgOfzud7+zBQsW6FnPnz9fr6V3QSc1MaJwURS9+OJ1In3W0z3r2YQDaTmBTcIGxh0yZkNw0gX+5HL23ve+1379619bZsu6C4oEZUCP+CwWFFRNAgIELUmNkg/yC3YVB6/aHbXGhkZbcuIJYsP88ze+obo2P+fimhubBLm+/oeXtePnzJ3ndeK2NkXtdXWgdAM68ShO8XB5aCwOzX0e3abOWRWHYOb4BGeEijiNVblK+9mvfmfPfOP7LiuuWINWq1q74pJzlCU49s/UKm8I5YuNRHDpKaW3j+VpkEilUzYAnT/4YQ1CTNOriYNA2PgdlULTtKmY8Z4rc4YyMDCmVmlwKnhFFB9FG5nuoSGdcmIfPjMCOw4SGEfEFqxFYChYTDYk+sNSJEupM5uGU87mYkPx5VIxno3xfKlUCrm7beMVRXWKpKiWF7vSlHetjAwNe5cpxY3UKDk6NqICBf6VEmVXT7ebqrq6ks/B17zx2uu2aNEi6zp8QAtOVK+IHV6czJM3aipTqHH/xRc7GdE/brC+vtF3bOpmxdqoKpZQLJC+3a+/Zffc94SnYEp1WPgaO//zn9am6uvrtWUnL7O+fvrwHH3ErXCyiFmGR3zYMf0vge4pVshmlbLxoFg0ngMPlX+THeCKGuvqU97tDJ3pCWrt1Md94pboWKl3TmlYCqSxKirjJiYQ78l990GBIzDDNaFUUkWxaqbeLiJnoWDHu7ttlIENCbPn+fNe2igJ/Yu/x/eV7ma8Uph59I71iuoxXYJqCVwgJPb3loR5hwaH/lPbNDm8LECuPOXUTvUhuuehMsWZhwKGT7GGUFC4dch0UCiYnrZFixcrTeRm65qa/T114jw7EFN3xDdepEDUrQnIGpo8P+W9D3X12l13f9EFHBLwAfNlw4YV1tfnwBInWxTwXKVONy6GB0KARCmY6BkiZXtHux3Yu89bk2ZF3XFqA6lkk6qZos6DUfRllXINDft9oGeT3Bvv5QIJ7vOVMZGTj4zIDQR0G3FMUNtb2to9xUaGvabG2tpaUg9jTgeJg8nPAbckHZtIGuSZpGz+5RtKI1nT9agY9MW7bxQDh2I+vp03Y4FIT6Sn1tMrvx4dMyw6YAonulDEV8OQpeFwyoZh7wD0JNVHTKxGh4F5T3jk76bc+fhcKEFOV1e3zV20yF5/7TVra2lNPpLFB+BgFq0PG3D2al4na2IqjdwqFm1wrGDbdz7glOM0mQGLtOLai8TKxczjUvbt22fz5813AEO9Zk5oyDGWVFQpD8gIpvCVjkm4v44giWcDs1gyY2lapSt8AvBM6V4HBgZF/Y7TzObGYp104ol28JCPMvMEpCjAiwBOzzxZADbHsmXL7ODhIzLdYPRsVKTZOfEgkDzXqCdESqjq33RBPzv99NPlPl555VWflVeeJlNZRplY5skHNhWZ3X5w337VdwFROPljI/gCKMyubQe9mWIGN8eFUd3iQo8cPqIFBIgJuhTpAj9jgUhH4KHNLlQM0ueeWLv4IoI790e0ZdUpz/Sghn5296XkufhbfBQ3XyEKlgrRNjA0bHfc+VjqX/dCECfkkkv/0UuUkC2ItDUPjyjegy2weqwHWDhVPRYo6GROpXZBBixE4ApE1ELIcj7eFGtB4DU+MaZshw3Ha7B6vI4xqd3Hj5fMNRaD58f7RyoWMK2eX3m5pmxj6mlYIZClfqLIvTwj9PGV3X9Q8ByQeBworFkmETKGhgeEFH70b/5ve+WVPyjOwRKQdqq6+aV7b1JExFA+ThW+Avwa0uNbb71V0nalGAIRAL8DnYoNwEVxkpwckU8ivFm9BynOosULhVcP9PVrE4AVYKIo1/Ilc79okS4KdM3fF1yd0qVTukh9hEgBJKX5N/hsGh85daSU5RU523TLXV7ISHAm17N8+ee1gQjIdJLLoHwPWVNrs9OnoECNg3Hn9XnBrxNil8yyePXFokypQ8KO1g0yb0aTKpzsSNArOLYwYVXM8ZNoErJsY4oTsKq4Ew1KTPIuXFdYPtfZcUAM9yRO/8iwm+k0hgW1UVf28InaYY3405FIpnJ6O/fChfM1WetY93H78Ic/JGyGQ0j8w3VnvnzfzZpJozr05KTKosLAJ6EF9WsRPQqusDmdXjsHBZLPVOHAmzD49wknnKBAqm+AzeCFUzYF74OvB3fHPNU3NmjHHj58SJuFgUR8fmDtRNzk69wQn8vCn3rqyVrY3/3mt7ppzLI49pr5WrCtux71lqfU5oiPX778ApueZpqFyarMaW93WlW6J6BZTljQjtU7l+bJKU1i/HdquCC1YvHJrUVSUarkEjBu9oFq6eLxfJ8TqxSO/rnBQVGnAaWcdeMkFlkVJlkeOpKmZHvAhyHTJkqoJZ/rC+uEjEA0eU3w6LznYcqytLEVCiLWiOGUMd1zjHANelbm649tK2LKtFBJBgSTD/qEmYcASSBDdMzDBDtXVwupwZDj95wW0gsRKnI523dgv33gAx+wg0otZtIJV7V2UQNep+ieIcOkbYqUY+eip+NdIJHiUUNXIwUnPJWBMeH1TU1Ka7bufMS5ZIlszLVecMFnLFdZptFkkkPNuKIXlTjvGBrzGnU265y3JIyAb4+/q+w5ewxZDERQT2G9FpJoHXEjVdVE+vBytNKzEa9A8miF5kFrS6eeXFs+e9QXvKWlKU3HTouMRKoCYub8EARSLPLSclTrWFzAL1Gp4RFMOL2d95Vu0ZQHkVFj8EOTdSIGIAzUIC5q6dIThfkeO9ZtrW2tCqzA6WUVYp5qIuydcMJJtm/vXsGMXr50rRwujJtvbW6Rn2GYMKeEoGg2jEjMgCUQSlbFn34CeWjE54HbRx09KmMsWrQIEfw1NzfZhk33KkZJDWtWna+0Ky+/yArTY3bayafZ7t27dQ3KsS2NRkuEC31+0ujFtQB98llt7e22f98+neQ4XeIMJhPPQgCB4sJefWW38nEYRF4hdE49G5WF4P34s7Ozs4QlsKHkgoRquuVUrj86at3dXcIgnBQCv69OmxP8JBRLmNHHsw7Xi/VlMxIL0a0r2HZkLE3ldqSRz+E6M4/fs0GmvhJcuhzpLm+KBIXjwR/rOip8ndmsPCA8F5RnLrK3p09+n5vid1h4/mRXcZMEJVJpSpuKG+Xhc+EgVSBp+HdV2sYci4cRo9NS7Qxebgy3EOlUwKaoSjj6VWZz5nTY6ut3ajChu+FpKUlcdvH5lqs0Wzhvod4Hl8P/pHf4dnw+zJuu7m49JK7t8KFDRrDLn+oM8qPq6Bh074YGReKwd3SKUtqUKy8T0tjS1KDnxGZQYWaqIFOvAk4isi5e7OVhfs5zBDDzlBCh5xG5ymgSZfGpYbiuDfGFN65geTvnzdV1URmlkMbJ5/V8Vv+gB4gEyzzv/v5eXZMX0fos8/hd16uLmh1K/k6q45Qd998hPBQSH1zsgUOH9YFwvoQNDw9qIXmo3CSRrgMLznFTE0SxqEieDwU7P+2005ReschRueJ3Gpsa9CAYMBiVpYghlPfWeQziIIr3qhFNf/FL37Lu3gGN5NCEiVzOVq+63MYV2HlxRtBdkl/DuolnNz5uy04+WYEsmwMkrSTHopGiruilzCXBrYoLkmvUYWDTV5QLJm2sdx4iETZgEQ9atXTIGslP63SDDPb36Rr4t/x91nsTCaSPH+9RysnP+CKdw18oOG1qVpoLMQX2sFrNAvXLlidhSA9EuTbdV1LRBK+ZN3++Zb5453qNJglcmoALKBUT3N8/oMUMhg5+ROVWsWkdcePGYZLyxckFatzz+htJF29cpr2hsUkLD6QIGkdEzOsw4SwqlTEu3OFFpx+B2Olk5fOCH3kdOW0ENjz8qPVjcVj4o909CmYwr6SUVy+/wIY0r86HJQDv8loRQFP/GVbjlFNOsV/+8pfaLIEQirac0sj4XnDxFBWnDhkwdbFsUutXZwdwdFdpkUOdCnUQUctQDUsR/rGuY7oHClq8jnEr/Ly7p8eWLVuqg6EYJCFydQlt1ABFla3x/04Jw1KiJ3Dg4EEVYYjRgqcYAR0HD26j+PWP3HZdkXIlUXx0XvDQBgcGBXzgD+YBeowSJdYpNaqpd9UMomi1W/X3yULIVShSLZeZyedrZaZggAqwSDNiRsZGZbpY6JNOOslee+01ZQQUQyicvP766+n389ooLHy4iKAzcVNBGmHzPfH179qbbx0QCdPVovK2/LKzrTA2ac0tDTrZCxYutD1vvKGS6FuJ78/G5CF55uINCxFb8D3BrhMTdvKyZfby7t0lBg3Xz7VF0AYjh40xt7ND18/p1eZJaKHLrngJl3QVi7d37z4vswJIqWbP73gAzPOL6hqDk72+79mAtHlF1/LFfdfpp9vLL79sdfUNSuUIltn9vCYsYxwULI827m03XV6UGTSmOfbLj0SPHHktfie6QgFYSLWYncb38IEnnniiHT54wJYuPUk3jAkiAkdJGk1WPmTu/Hm6gFdf+YNuCBkx0g0elDhwSVQAHxQRaNCTeFj8bgR4InqmICjydn722JPP2t69B0XChEgBVezq5edq4Wtq/DMwr4J5wctpDKUMevRoKSJHn0YpHOzXRMNS/AOBIaGSLBTXwCmlhkA0r5gEhJD4ZWjAq4h5ytfHpQg2o28LXa22VE2TC1Cw6ILIuFYWnqZLDpqKZJmM+A5Y2qVLl1lbW7v9fvfLugZa0kBbeR8KbFgv6OgLFsy3ffv26nPASThYUeDRCFa1UG25poheLaeeKD4wXo0T08NCCWtMgYMP55vWCBE1WKZmymmEjxgSkPdZsyBi4qGlliWoSywE9fz6hnpZADB3AidGjfUPDBr1gNjpgfJhbQQBq03awRlAkGh0ZDHxo2WZCvvmd79vv3zxZXHKYdYCb1512XmWLfrkCLmmRElSPSHx491v+8PgRPGemHwCOSzNbJ8vcIh2KLV5eZ4PM1fl5rExzXg7uH+fglI2GP/GXLNp2GQqG6fBSNGHCLuI9q7ow2NDAYodOHjImpuaSvGGqF+ogNBJm2TbyPe5D96bTIwdxqYjHti/392nGFKDrunPa5llK32ie29dUSSvFfm+ucWOHT0s8QB2fwj1xWkTzxwevSpzMzIbUIx54+a2ZlGCqem3i5yRZqAxpntoUGkh/vTAoYMGpRvMnx3Z1wfu7L43SrpRP2YjCeYcn3SZlcRa5XNYiGE06spy9h8vvmTf/+G/C/yAZ1dbU2Vnf+aTlq9w5kyAUUDLasdGIjU1kODmRPzUTLnUHpZ8uNQvEnE0zCaY++EjR5KlchYwGQInv6ba4wi+x/1Qv4+NvGjRQuH/PEOuHatIDYMNzgKxgaLMirVgERU/JJYubOawklw7B4vf4X6Ih/hZBIsE0Pwu38NKidUEIol0HPf44PbVAnCii4P55OTumOkaATW0D3t0yf+cAhC81994w1E3RBCmXU6EDhnBqML3qyxfjVBCmTU1NSp9ES2bnH98rCRH4qVCJk95vRlfxHuRu3reXukl09QCxabDrImGVVll+/fvE3y7+4299vgTT0u8IauFr7ZLzv+MlaXxKVTBcC/CABI/X5Tkujo7dOigTjlwJ1aOzIbXhK4di0MPH0GbyItJ5NDr626psHJsRip8AEsLFiy03/zmRS3k29/+dqV6eu8JRBXrFZSxIKR2xC08B6hgArTGx/VZvAfvSdPo2962xPa8tTfFOs5o4pl4EDolCBpLRPEMXOOll36n5xcnPdwGyqWsRWbbugvVUEEKhQlBQlMPRHnhuI1PTAlp4jXC4EGOxD33Sc+8uQr7CdQJoqAujLZdSYVOKpI8cuSwAsXDR48IyGCnc4qJKagtc8qxKjRa8jvisA8Oq+yI9RBF+m1L7K29e62hrk6Vw9bmNqVik9Nltv1OKnSwSgtWV1NtV1z0Wf6hoBKzPFtiFPOIxUEMghNI8Id5F0rZ1CQSBEN8hQam6pznw4OJPu5ZTrOwWAAABvFJREFUTGDvIHROBfCYJEqgRNtsXII6CkFtczpkesEh+JMvTj6nSzP3VCHEZ494Kq1NjwrYkAYl8jwbG73rlWfMurBxJLyUAB1laalbCYvgKGWSgU+/l9l+/cVFpLkwt21trfIvqnc3NGiXAtzQphMa7ZxoatZAlbBOojLEQ+ADeRBcAOkaqYMHRpzgCQWCwqKtKL5Z+G8CSJBCHoT8N0SDnm6dlob6Rj3gI4eRP81aY1uL3r/ryFH9WZUDSCmz8SmzGzdvV9Mg9KeafM4uu+AzVsyWWbWUpt2PB4YOTCuzy8ad1TDJ94Jq3tFBQ4e7lEhf6d1z7MERShaH9yBd4/5h33JdsSFU+yZAG5sUlgDKScyDBaFphA2BWed5UzvH2vL5xFguFU9KPKxaw/HeHnvnO9+pcSxYXiy1KqkpLS5RvmYri6eFn03OEPSNjxdAAfOSC4S7pTbfKevp7VGKBuEShA5fGcIIAV2qNJoeaHdXl0622q5BqdTsT8BHKbU+FS/qrLe/z04++WQtPr/PotTVNSifR6eGWvKRw4fTA3YtWKLd4eFxa2pDdRN/6Pg7o8zkGianbMfOB2xkytUr3vOed9mH/sf7LFfmvWlsnkgh2XD8OzIIrAlLywOONDFSOR4498TrMZEshuoMtEez4JWV+v67z3iHDg3AixdVvPERq4e76pw7T344MqTFixfJXfG7x4/3yvJkyp2AEvgIm4nMig5dxz8G9WwCKY0iFu3nsjKTE3JP3O873vEOcfkWzsciHJAb4Xq4LjZV5s7NVxX5UHwPPogTTQ15/779DhXWNyilU5ExhgmlZgF2rwgEaUQJf8eEE8k6ScE7cpyPRp8d+Wmda8tHg37C9slJA1o8/YwzlGcTmLS3z9HD7ek5btlsTvPtcQ9DQyPCEQBlvI5g1j80Zt954Yc2p6PFFi5ot5amZsunFqpAwBSApdZh3pdNRZFHRNNUYAnXFVg69+DFEidYsrD4V96Lf3Pdbz91qcz1q6++6n15GhA8LkugBpMCJW+v2EEqpTNYm3loWEr7YskyRSs9D16HYASvI4/n8/k8ov5onuBzvf89uIbetctXXC8CDX64YA6TXeS9d45OGrUhJ1YoJowHQu7HLzQ1tSQz5PNWPJhw3pZy/ELBWaTqb3Mcm9ewu/g5fx8ZGnS2SL5G3ZpUjCIHp3BAIAN4I1p1olmJk1dWJloWppj3amlpSxOovd9eqhaa+Ybahte6OXHeIQOciYS3B5R8EcCSe3tFi8qYVx65F+IINgHXHac+ImbftB4xhzvq7JxnR48csSVvW2y/+MUvbPHCBXpf5upQZqbRI049+Ln4c5U5mzOnU00msHZEBqFRNV+tE8n6+Wn2AktM447NiushnuF68f1oBcxUL735MrKgzg5Suv26bz4jJGe4Rlk6miZZdGrF+DOUKKKYQD66YP5CmXmfHu2Nj/gYL0WaokgCQ1XUph0z5mHGqWEx0cKXJhEQYxrnIXp2InZwgbyO3yO9w6wRaFEDj5vmmubNW6A5LgRAMHz5OYvOaaUbd+68ufbS715S12N9nevToLXHfYHaqfxb6uwdV0ApBm0qnvCQhN+ndIx74Wfcc4g68vv4V1q3+KKoJe5bf58CrUWLF9jvX/q9vfvd77Gf//znej9cBfcWamCSXU2jzvH1WAbFRF1erGlqbhRtvafHadFhBaiJ4PP5fK6ntbU9PfdpweE8R3EUYCtPeqDKCef9sTqk6/xcXUNP3HdzkZSGU8cNR3QI4MIJoFIlKtE0rcXO62bXExEvmDvPiQzlTg6I4gUXyqnhRr1Jo09/Bh4gaDhNV+CU4tvhe+MigpoEygYqxfu4C6AChabulDZM6NFyoufPW2S7//BqqVWrrtaFF+hY5T0nJrwVKXJZpoY5ROqyZgI2YNGWO9jBZ6jXL6lhuTy74+xBjOT3+Z8TxLOb0+6Wq7mlMal4e4eu9/oPG2JEFLJACjHv3Bdw9euvv6YYQPFKuReX2Ozx/vxJ3ULo3OiwGik62zt0kHg9hTUsAxuUplfiJgFrYfKnJ62ttc06OjqV4jmHcdoyO2+6rAhIAbAC3iu0h2pRahkGWXPFZ4CC2pIejqDMcl8U/G5UzXhg7PJgfCiKT6adm1C78+SE0LtIMXpT+dWnS7nsGj8DSJJ4YqI6QzKMmXFhJicnaSHK+/yY9OCERasbZkhB5Eu//40eEE8rfDrXiRuJiN3h6Ua5HDD7mKnnCCSl0y69ln/zu17r9tHoqrZJ+AGk02vkyIuhvBF1dgQLuIbe4z0lxhKHQSVwMZCnbJA6SNKpjYIQh6e52Z/HokULlAIDu/K5R7uO6WBSyeTZxrWRfkd8BTfQp0zOVDsJ+v4/WJZZZ4vk0WIAAAAASUVORK5CYII="/>
+        <xdr:cNvPr id="16" name="AutoShape 8" descr="data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAH4AAACpCAYAAADtGIkfAAAgAElEQVR4Xoy9B5xkZZU+/NxbuarzdE9ghmECQ85REBQURER0EcOiIobVNbCGxV1Zlb9gWHPcNaC7ZteAeV0TuigrigTJGSaHzqm64q177/d7nvO+1TXjhq+VX/d0V9269z3vSc95znmDeM8v0iBXBPIFdLIV5MpHQl9paN//l6+p6Qn84qYb8fh0C/ONCHESIE6AqN1BHMdot9tI2hHSJMHfvuBsTE9PYcOGQxBkAoRpVt8DAGEYIpfLIo4TRFEbaQoEQaD/0jTVf/yZX9lsBplMFu12S6/zd2l/D9BqNTE0NKT3RFEH/HUripDJZPQzX5MkMVqtNjKZUNfgNYMgRBxFyOfzem8ul0MnjpDV++xT2lEbhXxePydJ0l2ZJOH92bWrCwsYHBxEgtieIYXWIghD7NyxA+vWrdP7/LNpqZEgRYQw5WcFuq+7H92JL/7oN4iRQavdRJQESHkdvp43zXtAqPsIwoz9Lg20hvy8OE3sd0kHnVYdmRR4/TlrsGHzIShmQwSd3T9Lg3wJcaEfmf71CDH8/1vwSGPc9F+/wV1b92GiGqERUeApkjhFq9XSwqdRB5kwwNUveZoWh/cSRTEenmjhqIMKKOQLXaF4IXMhuRm8wCmYTifWElEI2awJXgtoa6DXc9GiKNLfC4WCNh5/1+509Bn+q9PpIAxto/jP4PspeL6Oi1kqlbRBHn74IQwODWHVylW6Lu+hdyPaz3avS0tVlApF/RxmA91Txv2N10y4iXs2DBckoYJELQk+ifgwKTpJipmFRWzdtRdxkMFCE/jDn+7DUjOVUP3GS4MM78Z9PpAm/HsCrh+3kjYcYsSthhTwjecdjPUb16GUzyFo7fx5GlQGkR1ZiQSjyCQVJNSKNEQm5NI0uL1thdMiEPI7F8BWvV6r4ds//TkeH6+hHrURdfiB1LZI/4UIkEljvPXF5yFjSotWs45H907hsINWI05iLTQXmQu2YsUKUDBczGazgUKhqAWnJdDu5mJJw/zC2kW9heDDNptNXWdpaUmay/fZxuB/QCehZYm618tns3p/o9FAuVzWzybkRNeQ5gQBqtUq5mZntaEP3XIo+vv69DfejwkgQODuLUk67r6cNtIGJAnSBJifn9dreW96T5ggE4bI5mzT8TPnFmt4+PHtKA8MYs/EHAJa5CTA7Xc/iKUm7UkHtJeUU5gmiCmrGIhiW0d+ju4rTZC0KcMUf/XkMRx+xCbk+drFvb9Pk2I/qs0YhTiDXHMJmaSJfK6KrKxHKjMVZFPE5RFkBs+QMJfVLcUvf30jbn1sHLO1lsx9p5NIeFqUToww6eDvXnweb1M3045byCY5IJcijrzJ5AImKBaLWlgKkAvDf/dqqjf5XtDalE7j+Z2fy+sMDAxIUDTdFDq3MDfP0lJNz5TPF2SVKGhqJc0rtYXfqfVmIRJtBm+WeV95aovbQP5e+Ll8favdRl5uqI1s1txDQK2UVTBLwbXhpvPmWvcWxLrHMEy10WdmZvD49p1otGNkiyXsGp9F3GohXwTma21Umxk8+NhWtOIYowPDWDM6gHse2wagiKhjG5pOkMrEfyNqydS//IxRHH3sYcjRDV3zgY+klUoFU1NTyKQBchmglC9goD+LF55/LIbzixJ8JsigU8gju/J8hCltdtC1s61OHf/ybzdgz3yMatsEyC9qHn/OJAmuvuxp2Ll3L7Zt3YrNmzfioDVrzBXQLIY0uSZe+vp220wuzTW/+Jo4AIpJqof1LoEbI5PLaYNMTU3KHVTKJUTtSIKnkVpcXESYzWgD+c1CM9hstmTJKHh/v7wHCl4mmsIPAyzMzyPP+wiARqOJUqko7XdbH7EzqYVsQZvOW7Ukjc2sh1kkaYIwzwfMShHA2CPNIU4jPV8my+vxirYpOnGMhx57FAky+nwa93VrViMMUuwen8DCUoRCuSLXOr57CusPGcbCUoIbb3scsbM0iUx+jDjifXTQhyVcevpBOP7YI5Cjdfra93+cTk5OIZvPYXF2Dq1WHZ1mC83aEi668Ew8ZRMvkKATtVBZuw6obAJwsAu2nLTSGD//9S9x1+PjmKjTZ1mA4bUvm6b4+xedi3sffACDAwOYm52RgLm7qZGjoysUsMnP0i8FAbgZzbS7YCbsIBMtIc1YDOKDuXyxoJ/r9Tqq1UWUSyXEHXMfaWwWhM9GQVNb+RkdBXctFPMFZw32DyYtwMogl8mgVltCJpuRsKn9vGfeEy0X/TEFz/9nwxw6nagr+JSCp6Zn6EZChNkYxSjB1h/+AgPnn4MiN5CWzwJDfiaFVqvVkM/lUGs3MTs7q/UqlQoI6Q6RYseOPRgaGcHs4iJ27NiNeq2N4VWjCKI2vvrLe+UAJHSa+JhrEKPTbmEk38alpx2E4449HJk0QfCOD34kzYQZNFtNLRhVr6+QRy7I4PynHI/jBsaRBDk020sY3rQZcaUf2cxJ7qadEQ5Mw7/89e/gvskFNNsddCLz9RRAFhHeetkzcMedt6Ovrw+7duzEMcccI+HXanUJmQLx36npWgi3CWgRGlOPopx+G8mKd7hg0KL+TC4rTeQmu+22P+KUk09BTjEBfawFiabRAcplBmyJgj0KfqBc0bVCxg30i4r/GEMkev4AKVrtlhbcgsUIWZnkEI12w3Q0yaGDBKWcuRMf/EnwykKyCOlKqNWdNh79yBew+nUv12sz2by0ks/HTfOlL/4Lzj77LKxcOYpyJY9cJq+sIuq0XWzEOCdFua+CyalJHLJ2LRYbEXbu2YeJyVk8vGMav3lwL8K4DoQ5cylUgqiDVaU2XnTWRmzZvB6gqX/Lu96tfddxfpVBRtxsYMuG9TjkkEOwAtM47pAYzVaKVUccDpQqCDIbkIYruhE1nODrrSo+8cUfYu98FREFrwAjQSGu400vfibuvudupTrc0f19/RI0NZWawZ0+NjaKYrHkAjgL5LiQXPBcPo9Mu4qwOOjMv5QQoYvwd+zYidnZGQwPDWPzpk363Hq9oVSNLoAmPJfLY/v2bZhfXER/fz+2bNxk6ZpiAKDdifDJb/wSrX33YsXgEAYH+7VBR8dGkQYBRkZG5AYp+HZswhifGUchl8FAedRlCpa5cHEVIHJzcrMkKZoZoDYxhU6mgAwySNKONhQ3CTfiXXfejqOOOlKbJJ/PoL/Sp+C31WxZzBGYBeOO4vfFhSrmag1MTM4pGJycmMSP/vgomkwL40Qug66FmdWmkSxedPZGrD94NeK4jeA1V70t7fo4mp2UMVeMSy65CFOT0+jEAR579HE866zNOOWofgSFQYSVAoLcJgTpMJIgRqCcn0Jq45Zbb8cPb74X1VaLKaQWYTDTxute+EzUmnVF6ktVi7Z37NiBww8/HIWCBWC9QqcGc+GoEbx2LhMqIOPvvannxmCEzvu/7757sbhYVZ59+mmn6TWNVltWI+lESs8ovPvvu0+awLs9+sgjZL658crlCh7cuQ8f/Pb9uPJpwxgaGMTu3bt0X6vXrMGGTRtldnPZnEy/rpsk+PUTX8KmwnOwbk0/skFemRAjfL6v2WigzRRRAVyAb/3bN7B+06FoNprIFYq63pFHHYn60pI28ezsJFaMjiBIEzA2NHdYQLvTRtzpoES3FobIZ/Nah4WFRSzUm3j0iZ2oVhuoN5r4/UO7MbOUIHJ5fNrpIG5GOPfoEZx34joMDw8giSMEL3/jW1Lmf0p5GNgAGKoU8IJLn4PFhTrjEH3Iw48+imIY4ZXPPQKVTBXIZpDk1yE3cjLSJI8gJKDCuH0JH/rcd7BzugFaKKYTo6UAr7rk6Wi2qIFZmTVqH687NzdrQVmlguFh+m8LvJjSTExMaAE3bNigTKJSKTvfYj6RWkCgghbhN7/5DdasWYMjDj9cWsznec+n78RVf30csi7Fmp6dxbZt2+S7+d7jjz3GNkFAN1DGzp3bsXdqHpkkUrBLa8QgkYIfWbFC1oqWwjIASxt/PfV5bK6eg77RMdTm5pANs9rU3EzNVgsbN2xQlL5z507s2bsX+UJZcU2xVEa+kMehhx6K+lJVlmmxOodyOY8iQSKmtKHhE8wQCsUC6JK56bKZrCxBbamBbbv2YGJmEVGUYGZuHg/smsPjuxgQZtGJmR01iTzh5ecfipMPX60MJqHGv/T1f5MqCGDixwgzAM44+TgcfdTh+NOf7kMUmy9dvWY1JidnMTG1B1f+xVEYqt2PTjNC/3FPQWbkFAQMurjL0EBUn8XVn/oZlhqUfILNa4bx/HNP1s3uZ6eVH0vWWkjmt6NjY2g06hgfn8CePXtw+umnC/EbHRntWgYfnevtYYg/3vZH7Nu3D+vXr8eJJ5wgMyNrkBIPyCKJIgnxlj/8QUIblhkfxNFHHWnoYpxICLV6DVMzM6gtLEqo2VxOm4jBICP7NavXoFwpy6r4lOy+Jx7AVP4OtKt1HDN4EVavXG2pXauFdquFSl+ffvaYAnEOC+kYzWcl8Fp1Ud/n52cQZlJUaJ06bX3G4OAACnlmL4w5LPenJSDwMzk9h30T01hqJVhcrGF8cgq3P7wLaVBEGrcw2D+ING6inM/gvFPWY/3YANI4EpoXvPi1b0gVfSaxfEIuCHDB08/C6NAQaswj832YmJzA1MQEVq1cqZ3M6PySsw7HxuqvcfBp5wLZPLKrTgXKa5nEIY2X8MjjM/j4N25Gp5PijKNW45xTjrHgURmmhyzNT/svRvaz83PSKm4ELiDTNAaAK0dHLUVzUK5/D9Gr399yCwYG++X3DtuyRWkU79NchWUY//7vP0EUd1Cv1zDYP4CnPOUpyiYoeCKJDPwWFxcU+XNDcSP4qJt4ALV21SoKNZR18HDw4vwCwlIOeRCCphu2TdeOLYAsl/oUv/B9yjSE5Pn9bz8060tKjaNmA5kcIe+m5FEp5DA6MqwUVprPjZjNal0InO0dn8DiUh3bd41jZmZOIE0rTvDYIw+jkxIW5/qmmJlbxBuveC5WDPUjAP1vB8FLXnsl41kkxMi5C9MYFzz9yRjs68PIyoPw3e//BzZs2IhDN29CjYjS3Bymp/ZhamoGpx67BRcdsYS+0RGkURbZkTUIhtfL58edFn5ww0+wYwY49YQTsfagtUhSQqghgh7s3YMjFBQfqMHswqVhtADUFP5+zSoPmdqiefDE49U/+tEP8OxnPxv5XFYC88ieoYIJvvWtb6HWaMjMjgwN41nPehYKhZwEz6zANhtNo48tLLjsBYxmZmdRKpYk+IWFeW20pVYN/YVBBGmbS4rQSbUZtXXtSrlProvXYXyTybEWYICPNF/+nJrM7AIIMwSRAqFrvH4hl0Olr4yQbq3TkQvqRJHwiUa7hXY7xsTMLDpxCjrq3Xt2Y+v2HXh8zzxajRAnHbcF//mHu3DVZWdhzdgIQOyAgn/xq/86ZSrD3cE8cmSwgjNOPVFARTabx969M7jngYfR11/BYYceqhvs6yvj8ccex/S+Pdi0biVe+pQKiuWKHqCZFtC3+kiAaU4c4QvfugWnn36StJU5pfd/HrmSBXA4O39eqFZdsGXQKYMvoW8Cd3LL5qHnJ+HXjJwd2KN0zL2Wf7vpppvw2GOPKTikmTzuuOOwZcsW9Pf3KY1lbYGL3GzWXexBvD/X3aCG1IUuj7eoPopalm5mrEbA/6TRLjefXZiXxq8YGtFmaneIT1hsYM/sN1WAbIbWKVQAawheiDyBtEIO5WIBhUoRGVqiqI09u3ejVmtYLYM+P8xgYWlJiCQ3RL3Zxt7xSXzz5/diurpEDBdRJ8FVzz0MGzYejBzRUwr+Ra96dUp/YVqS4JgjDsWmQw6SqcvnCgizBfz+1rtRb9RQUjCyCZVyUbs+G7SRaczj2KE9GB4cRJhnKpZFFORRXrEJIQpYbLewb5GbyBbS4NP9v3o1a3xy0upVSYKxsTEtpNA9p+W9xRvTGHst/feTzzijK4ReTb355pu18ShcCpzvocaMrliJhx95GIcddqhuiJAufa3/UnlC92z+la7QinCEf1vaXNS6YqHgAB3TYH72vfc/jF07d+Jp55wrX01s3XCJ5Y3iP4eCp0JRcQw5zCAfpig6wRcrRYT5HJJ2C1sffxyZXEHK4HEAru327dsFz/J384s1XPtPN6Da7iCKAuTTCK89fz0OPWIL8gqeawhe/TdvTGlOozhCmMQ46fijEMcRWq7QsXbtwSoQ0Fc1G3Xcc89d2gAEYsaGB3F05hEUC8BA/wDy5SKCXB5BNod6M8Dw6AYEuT5MN/Nox3l0gixCpEKOzF57HIi733zgdR/5uNIyBmMffc81KBWLLnWCgJCudXDYAS/zuc9dj5e//Ar5P7+JPOwqH9qkSWzJT1NYvHeLzjN44RWvxre+8gUhY9RMvzFlkVTBo3ZyMwQy3VbetZ/9a7278huR36uNJv54+20487TT9Fr/5QtNvJ6hkgmymUSCzGWySv0YzdNjlfM5rXWhUkCmkEentqQUOFfIo9mIUHHPkMmwfgCMj09qA9JFvulD30A7YqU0QSbo4BXnrMfhmw9W4Kilv/B5z025GOvWrlVAcfDa1ejvryh9mp2bRZxE6BCISc2sEKTsL1eUfo0M9ePQ1h0Y6K8oTy6UiwhzRJtyCIoVtNopBobXIghLePvHb8DehTb+8tLn4vgjN5omOcxbwhKgkeA1b/8AOiHTwgD/dPWVCAPnHhJfj/eVQds8fMhf//o/8bznXaJrMrWzwoyle94ieKEIPnUC5ee+7K+vxJev/2cBLMTK9xOig1It9bCSrxe2TwO9Zel1XYK4EeC+B+7HkVu2KENYtnQs1tiuN+g3RiFv0XpWpjsE91kuG0jwMvXlAggQRPUlaXa1XsPw0KiCPX6x8ENwaXpmBq1mW3HYWz78TTRbHcRRG/l8gsvPXodNB6/D8KALkJ/z/EvTgcE+HLppA4rFAlaODQk0YJCkuncUK9qtLi65Wm+iXDKfy2NkcAibc7sxEFRRYP7JSleGwVUWGZZTcwV00gwKfSMIikO4/LrvoFGrIwlYnkww2NePjetW44Lzn4Yth6zDJ6//Mh7dPQ7kCtoI1175SgyVgLjREkKnyJZAKgkU4H1VMbhiGPNzCxjq7/szF+Kj+t4/eEFp6VPgjf/w//Cpj7wfiCPVnVi4sYoagSl7J7+FQQatqOW0ny9nqhjYexwxQ9kRU9ogRKsd4Ikd2+Q2ezV++V6MEEIrUypmtFnzJEi4cnM+E5hlLRaQKxPCjtGq1bFt+3ZkCzlQy5tNuqYsgjCLUqmCMJNDNpfFtq3b8I4PfQHVdgYED1fkU1xw8lqs33AQBomM8tkvu+Kl6dp1q7FuzRoMDvQpcFMli/wOmjWmBQxsmg3ML8wrNWm1Y5nKfBhg3Wg/VlbvRLaYRblS0aLxBmju+RC5Yh+QZJAvD2O82Ye//8x/oBU1EGYI+ph5lwYSnQpyAjYCFm8yKY5auwrFTIJmdQnPe9bTtdkCvjYT4t0f+xz27NmNv7jwAlx0wTnIWu7lavWe1cPCiVUAewUuoVNoCPG17/8HfnrLHei0G8jEEforZRxzxGY8/aln47CN683KxTHe+9FP4pqr3uSw9VAFIC6gIfIGTfOzmOb9/k/34f7Hd+D8M5+EjesZpyxXLL3lYebCzUXLUSnnpGw5MpPCjKGY2UD5e4WxVoUwbQeNpSoeeuRhlPv6FHizFkJLiyCHThRjaHgEYdYRWDJZdBAik3Z0j1a0S5D4MvGr/+av0vUHr8f61atlvivlfJd+ZP7NLsSImNt7sbqoaJVwJMuEQ5UK1jbuRCYXWuUqzzwzQMjiX5hBm/VUokhBHmvWH4of/G4r/uO27dpYbW4qMEJuW82fhZT+QcGwjNL5+7hZQ9xuId9ewrVvfS1ymQI+/vkv4eFd4+4+aWEiHLpuFd706ivQV3CEiwTohFZmpZCotywtKyf2QSECXPPxz2PP1Jxpdmo0MRIzGGN0WE7lrbCQggBf/uS7tUlrrOk7nMCTKch5EXMoCfHCt7xL5eIrX/YSrBstY3Z6BgN9BdUuKIRGo4Xdu8exa/dOvPB5F2KgXEahyHWzjIHxbzEXopjPolzIIlcqIUg6aDWXcN999yNXLiIT5pB1sVcmVxGoVF2qyn1QcbmpGezJUjIY9eCZMznB31z1uvToo47C6NCIBJ/PmW/0VS2PmXMn+jIq38uSIdOf1cEsGrvuwPCKYb2n1N8H1qLDIMekFDFyKBT7URwYQTbH2AG47ut/xI5FFnEIJpgtJZbA6DTPYM5CeTFWmAlk00Rwbzlp4bCDBvGH+7eDdLFcPsccVItJGJiVqDBu4Z1vfT0OWTmCX9z8R9x88+3YO79g1y8W0CYvkFS0NEGGcUsh362tJ6nxANBuyVfyXgnEEOPnfeTiOlqdWEAUOQkK1LKM6Gm1DIXMs9LJIkyWVTWWsyNRusJOAykrZtT0hG4kRSZMcP27r8Lw0ADyBa45sX76+ACFLE19TqhbtmAaPzW5TzB2QjdQLIPgVS5bRCZrha35+TndA91th7uMMQq5BdmsXJLnMcgCXv3Ov01POP4E9A/0qUzpmSI+L2XgoAjZ8ceIGQ8OjSDMpajNTCC751YsTe+WyeEN5ooFpAysuG2zBWRyZWRyJYT5MoqlfoRhFnGYw1VfuAW1CLpBCo4mnOaOJsyDebwHkidZQ0ijlrFhWGpkvuwCIZp9sktYcTKwhiRP4u+GS/B31A5FzTkSOwzdEsMna+VfQruMri11C7nGiNp1wdc0xdyE/EyRJDr2OX4RubAiXDhCYTZfVArMjED3w43SInBl+TtfqwJP3AFD5X++5rUYGBg03oDz8Uzr8rkMSrksysUssvmsyBSsMywsVeWCc7miaFf86L6hYQWM5CNQu8WFSN3n0fX2pNDdNPcfP/Cu9Oijj0bfQAVFLnpgCJonUdCP6I3coSI65rBipB/ZzhxytX2IOouo7duL6clxjK0cQ4YFCNa9aSZzXARWxXISfC5fRqFAn5TBTKeED33vbrFd6Q2I8qt2DeKelrrJF4fmn5NO0y28ESy4g1ms4AMGcYo0dsGW6E0mSNYJjD3kijq5vOruZAGrPiC+Gz8nNMzesWnQiUU8YZbD12nzOOSMfpkBmQiNciEeRXS8O2U+WQQutYxliex++NncuAS2WDEMgwSf+ofXYHhkRByCbM7cFO+3kM9K8KWC/Z4b7oEHHkA7jkX+LJcHuDgqjBl7LUB1adEwEJZkewTfi5P4+w2++rXr01WrV4vlwaqV1ziCFdqhpOrStBGhCjMkD2HjaFu8vGa9jrjdRNysYs9jD2JguB8ZmuACNZ10JQYreaRBCWE2L7+XLw0gn+tDjDZ+c/du/OC+mvBjZlOMSOlDpXUUvMyhOSWaRgrn0IP6sXXfEpKQ6R+lZygYo3wKRCogjXRsU2k8HTWZKYzWtR+M/0ZPyOditcuBWKxokc2ijeBJoEnarfi1Wg0XD9iG7AaOzl0pLuKzhgy+YrRbNbMQ3Ci0KjT9LuAM0wiffsdfYWCgT4hhzmt8wOAui3whlLknqBS12rjznrtQHuzH4OCQTDyYriZAo93R91p9SXEXuX9MSRhBJQ5V7Kad+n2A4Mc/+U5KQCOXz4hkwN3vH0j+nTCj427HaQfFxm5k2nPYsPEQRMSK63VE7Rr2Pf4QKgMVJEEWBW5ZMkizOSAoSvgQm4QBSQkD/YMIM+TlRPjkz7Zh20wTqk7QVwZMVag1zu+H1CQgK9Od4NzjNuC3D+xyTGBHLdZdG3tIbF2nkWTL2LMAMS1DYAJmakaBRdwkjCXSZZKmuAmuTE36uEyzYyZRGXRtugrHCtbN9RSaqIXc+Lwjlpup8ZaimZknN5/aLvgaMT76lpeif8BKtdzkSlkp+FwW+XwokkcumxEWQB4e01fB3glzfqDFmCXOY3qpij2zc5iYmRNPj7WCyZlFTE3PaN2EzjLnT0l3zyC48Vc/Tum3izkLSLxv5wsZFPDqeQoOQH3mUQwkS4iSNhb2PobDjzsJcZpFVF/Avom9QGkE+8IxzHcsKm52OjK7LIIwJ+bNczGYEkqzyRlfrKoQwyCKpVLyyK3yFWL16tWCbVetWiWK0Y7tE2i3UmTDMgiRkGxA16SFdSVaU2fXTOCid5pDWS9uD2/JaBIpdPpD+VwK1Qo6PjXzDFlqqzYV1yS0ErIIoO493WvyNY73T+toG8SII8IFGE+0m+b34wh92Rj/+IbLMDRQUVWQ68/r5sIApTwFTnOfU7DXaNZw74MPYcXQCmT7BjDZifGr/7odv/j5r7CwuKh7bjZaiq083Zv3q/RQjSP2DFIoupxb/vDrlB9AOpQ3W3yDSrREk/IFFLIhGgsz6M83sDQzjrSzhKWp3WB4Mrn6RDyydwaTM7NYmJ4WLNpqkDHCsqpl1wGjJUdOZIzAxgOqCYMaMlomJicRODIGF4qfS0TO4EvL9WnGy+VB9I0MYGx0NTYefgRWrdmARx7eiUZEDJ3mXi0SXcFzc7HkaigZwRZWDU1oKrSoGhd3N4AyBLo2x67hhvELpss6gEaBo29scBU2a6rgpjMLqTuReTerwcIIf8fYQTy4pIOV/UW84xUXm+ALRgRlbJPNBMrj89kcClTGDNCoV/HYvgmMHH0qrv+3b+Kmn/wUzaUakpibqS16FtNgGnLdpweedE1bG/8l2Pu2229OuSuIEgmWJFWnY61D9LnFfBHtZhXlPJDEVTSJ4i1MYms8jDu27sbM9CTI0m3WG8rzSXpQaZJa6FKIgCkSF5sgBzlkDeuCUTqmbhLyAai9xgX3xAziBTSBSptUuOH9RdIkslsYMwyvXIGD1q3H0aeciU6SwfT0IoKYKZsBJGCwaF5N2YMv+lBI0liCMNRALprzvd02JII0PW1cerFr6uBr+JV4eM9bFwnb/KhF/wbskC9HgXdY/ubnJh0cubYff/OXF6GvUjIGsKvO0UUJwMmhtTQAACAASURBVMnS7zM/A+qDa/GjO+/Ad7/4RSxOT6M6tyRhE71jzKB7UZxhULDhLz2Bp3sOX/0L/njbzSkrcTmmR2J0UvAdVYoYZbcaTRy0ZhSt9hLSxhyqrQQ/fGQntj7+BHbu2KViDh8iH2bRYTWo1VavF4kN9CX+i5pLIERmNKILMHap98Eyxu5GuVA+q+DfvQYyWOli4u5B+HTtVhv5QgnDB43h8GOPw4bNR2PX3mmkCWlGXATD9wn3d3NZ19JkqRU1uCPfq9cR/OFiOizBP4OYSq5nwN+HzwR8XYBK7zeUrbxzEdlQkCvXlqkc1+ysI1fiZRefp3o7LS7jWaGdxEyyxO/p5/OYHjgIn//eDbjlxz9WQN1qNlBfaqJea1hmwazF1ROM9r1MF19Wc2cRfX3k97felAouDPkhbDeyBgfGZwsLCzh43TraAbSjOqr1Or53z0N47MGHsG96EvW5qpkR+lpqRxoKsFhYnFckOjRozYsKimxFtC1ljrgBGEGLlNhCqVDosm60GZyvtZ1sixfzvU6jFMn3PCT3GO89E2aRKRVxzMkn4fjTnopHH92joE60aaVUbocpTTOzTpaQNmTbCBPmmy1OULDnzCbvn7IkV4GsIAV+jlhpG8HKjbpfFzjK1MsCpOqGMaoXsYEEr3j2GTjz6E2oVAhG5RWRM0dnUpvPBsrfp4fX4Gs//BF+8Z1v63lb1RqYWSxVG0g6ZlloKUzY5t+9lRKwxKyFn66mFXNxMvW33/m7VACNfEtGwdxAqYJGbQnDI/2Wr6YdAS3fvO123HHbXZidmUCtWrWOGknGkSmcxs7PzWgB+ojiuQVQlbOnGdIvKv9OCJMwr1AnSlDWzW7UUDHv5ykkBkl6TMtZXb+sqMxOQ/3DFQf7cNqZT8bw6i0Yn6wJE0ji5cWhn+X1fDCXOFPPq1PjPa/fkD7g4tMOw3Aphxt++wCa7Eejm0jNaoWsx9HfuoYNWgLhDS4IzKYBWu2aijtJRFcX4W1XXIzD1q1EX39ZcY1RpcgoNnpVe916fOM3v8F3P/tZ1BaqhgoyaK7VQeNET8brdxtCVX1ZFrA2rCd8sMdOWY6hecG2HQ+nytPNXuDxJ57A0YcfoXowIUxT1A4e2LMLN/z2Fuza+oTo0Z1WJLSNC5QLrSDDYExtU0xX2EjhCjVSBEGvy3mPj4yJhjEIpPb5WrUE3omF5JnGEZQx7bTXE41yLdRsfHAVLW/GTUUNDczm81ixcgVOOvNszNbLruHTbyrfsGnBIz/TbzSfx1twB1TyKT74mmcp335g6y58/IbfWZSeWPA0UExx9tGbMTg0ALJvdkzXcPeje9FJXJFILeANtJsNVQJzYYLrXvd8rBoZRH9f2bh0LgilArI28rXHHsO3P3s9gnobs9UF631okyzJFJNt07auXmFo0cTjd7QuAW8eCEnNTbJ2IcewbeuDMn584F27t+PILWSjLGtbSsJDp4Mv/e5W3PmnP2FpsYrFuVlpL1E9+TYX6PhArN1q6Ca5YqwZq0ecrcmwuEFsWxclCxGLY3HLuNhWwrTAiF/LdW+XirkHUBqnaot1wfhWKh9t+9hAGiQwpIC1h23E5iPOxkw1Ul4fKge21IqWjXi/zGVkm4zBqQI0JHjds0/BiUdsEMBF3ttbPvNTcQUOO2gIVz7/PAz0FY1k4hDHWr2O93zlF3hk15Q2ra4dR4rASW8uFXO47lUXqWuGtHFDLRkQk4oVYm5sNf7hfe/B1ONPoF5toLG4hEg0MWtKZdm6G++4YpoXfJeswt/njJwiM2+9WsaDePSRe9K5+XmsX7MGCCx/FnTioMqApcMgwAd+8GPsfvwJzM3MoN2oi03q4dzeHnANFiCCRi3nYjKQ4W5nBymBA0er9bvS/5uoIXljZMowyzDs3ARP7fZt5f6BfdVQ+DbNGbn0Dnvw1/RWhdaHPpQo0Nia1TjhjAswOWtAjG16mnWn9Ywj4tRtVFcoCgNc9+Iz0NdP1GxYz/APn/gOLnv2Kdi4akiVSNKoSZfig6saFkW48iNfxu6ZljYPg150Wog7LP7EKJWL+H8vvxCrVq2Uj1ddnSRMRuO5DH40OYWvffjDyKUhlhZrmJ+ZU3Acta0TNqZ/d5aOz6D18B7Qde/qn+x/cJCzBG/BAIId2+53Pt7Ff0w7HFNUQUkSoBp38I7PfwFRvan8ul23smTiWpx1QZcoehCIQmfpVakSc2kGLs6HEV4VE0abzOWdaqNqSPs8iMRqYLPe7sKdPupXHaDXnCk1dJvK5azd6N3FCXzkTDY0GHRwAOdc9Jd4YjvhYm4qq6AJ+KHQ9R/dHwXPew9w7UvPRH9lQIUUami7k8itsXTKz+qrlJV6Gb0a4iy88rp/xXStZe1EHSvwsGWZ3/vKeVz3hhdibGRIVVG5L7c+gysPwT/dehN+8JnP6P6qMwtoLbHjJ2PDHshWcmml4hkH0BizyBWaHALLTKZbZHOMJHEHd+14kFVHV6PmbjI/4YVPwd83PYWPff5fZY7n5+ZkchTYREZGoKaxYCKBqJKX0YL5luGUwxKSjh7MdhzfZ2M7WEnTZ6n6xc+3yNkHcHFkkasEaVmquXBXePGbRDEhNcBPvnCsV6/9phXcIHI4GFq1CqefdwG2b20gn83gnGMPkRn/7n/dxZKhLayvwgXAu192FsrFigRPIVHgCgLZxMh6OmOOuC0XwveOT8/gTf/8E3EXhAa2WNjpICVyl3YwUAxx7etfqALNgOfOuecc2nQMPvbv38RP/vXLlAZm9hHgksd1LsjRz3rmAsiUZ4ysaWtlcDV9vA98icR2K5+7dz6QygcIraLf7MV4yBMP8YddO3D9176h/LK2uIimIw9GrUj1cC6l0DUKm4tSKNrCEaZkBCn/Sf5XR68hN73XHHOz1KqkdrnUR8iYE7KCq9AKHMs7Qu/3voubVQ/sQRS3v2je/UQMml5x113vO987vGoYz3nui5GPs3jSYSsxumIIP7nlQfz89ifkl3NphNEVfQg6EV777FPEFciRaCJuQkEAlPAOdSDF6sSp1uoWOacpds/U8Jnv/Qbjc0TW2GjSRqfFGT8RBgvAu15Hwa/A0EC/TcfgtqcVXHsoXnf1mzG5fatKzlN7JtHh3IGOwcm+zNoVLhXJTwhxZFDx7DXQwp7ZK7JiCf6egtcOcRUkXwZ1ayfB/+qhB/HV730fGbJLG03l96VyWRE/YUMPanAgAS9M02XRsHWMdtqRmjFs8gQrgMbn4xdNF+MC+kDW232TJFXarsF766mC9RAlfflYZt5tPrZNd+MIEhBcOsWF55qqGOKsAu3Ohk3r8fn3XgeNYBChsw0aeQFMCjzbyDgcgDV1wxCdFWIwB7aBM8hNMTXJoQVVDV/Khnm0GzU8MVnFxFwTESNql3qxBFUuhDjs4DH10omHILIlkC2vwOLAClzygov07/pCFZ1mB20Ol2p7opdLZl1G42XmgzplG07wHAph7CbPHbQAO9i9/T4J3hcTlArqhYa6Maj/z4fux5e/+31ZBX6xyCL+eQx1frL/2uBJE1CxaItLTp5cAtOwTgdlNxjIm+dljSWJoGpUoR6Dw3TQz74hgdP8mQV9rO759mb/wIpJnCWggBmWW3rJoIj0Lr4vRSFfthjFggYce8KR+Ke3/r3VFBw6YN9tuJBCHocRMCAkoqaRCMp1m/pMVtHsy+BpFmvkXlzM0VvA6xZKHIrm75vSKY1swV21GVz5ssvlPmenpsCCe6tJi2kVSJE/3CaSiXdarfV0d2FO2PrzFN84S2DE0RDBrm33plbNMTOrFwtbtxunlm+dmsK7r79eo7zYfz49Pa0LksMWkbNOPyZcm5W1SIKXRlOQbvAAr1UgEcL5TW9R+JnUdGo+f2Z0T7fAtmUjL/ohRRYjdWnTLK0q1bL7VZroNibzYFW6OP6M07ESG8ZEU88qPI2z0kg+tWvHPvPME/G+173WWQubKME14OcRMeyicc6dMDKXSVfjlJl2GzbkNjvDFlcA8trWGzQ7jnVXG7VJMgWs2nQyfrvrYVzzt29WlD89OUX+F9qiSpu785u7m7Y5KrndiOvqcZiAXusKNZIZ14qbYPsTfzJT74TufYU3lwRdluIYV33sY9izaw9WjKyQORNAE2bEvo3qNk7MI2Z5ES4ziv797zTPxhcvyHdj2ZIkxowVaRrNpjB3sk206TizjTmcQ798dcsTNdQz59I3+XE/G8fh1EqpOJPGaYcWSUkE0zZHRhC1i6VMoNzfhysuex4uOpkNJS6ecOsiDXVAUrfjV1mLzQEy6Hg59LTgys3qcTvcv6Z7bTapOqSQm0XBbHkEJ552IX744O342LXv0maan5xGu2Fz+biBvUWWn3cWdVmbrTZgf7PmjO5XYAJn3CNTv/WxO/aL5gwNNRaMNgHBlzCDN33ww9ixcyf6Kn1inwqQcflqa8nmyfmgg2wer/FKP8IQfUxZAvpO02JW/riYziIKtrWCg2kaF0OQqcMCLE0xbdKmFI3bNpt2tcP0lwNEe61gaPc3EiK50RgzeOugZgfahlwGI6uGcd0rL8eqsgE3VoFzNWz304EIoyeKShP3Z2Toc+lQ7AeLDZQ1+c3gt0vQUUo2sPpobDzyqfjmrb/CZz/0QY1dmZ+YRrvZURWOFsBruy7hNJ2/M/KKZWTmEi2GkrZrjay+z79L45949Pb9BO/RnS7+y3AmCXHVJz+FHTt2mUA5k6bRQKlYUdNhxFzbTYOU5udC5IJQ06fYj81FZMrDpkBGwuz0ILmQr1XFS926ie1q23eiIkuPxKaxFE/+TNQsg2xlrknRJj6uoYVu0uMBdCNR8Xt64nxFjUGnf5+lPMARJxyGa156ETLUSEfA6DXRvaQLm79nFT1vgnutp35nXG5Xo3d7wAWtXY/sovK1R12MFasPwse/+Gn88IeMqYD5ySkkkbVs+U3vYyMGsvwitd1vCG/apRgug/EKwPsVY5iA138neAV33RZhUpECXPu5f8EjW7dK4H0D/TKRHkWrL9ZMu5wPCYwnpfStVMx3aT/lkk2x5AJzwyzn2AGWFmwciEG1ROIsImcngP8d8XTjsftq1HKRpGsJnDb5a+vhGR73jEZl4YJfrTpHlbQVRKnuEDeRLZbxgueci+c96ThZGwWBPdMovUXxwv4/v7Ms263ULTd2UOhe8N4qHHfmy9AulvDcv3yumjKrC1UsTs+ps9lrhH8uWVjH2OFoWD+mrbsONPU9FrHL//f4x4GC38+H6Kksgvz6D3+AX91+J/ZNTmPlihER9Kkt1NzZqTkJQ0T+lEOEbKJUg+PHOEdOXaaWRlhbVluRsebcudIqW6v4ZRUxC9i8pgkAcUQNPxOPVoAFE2M1G2BB089Ie7nO76ZfMo5wjFsjaFre6ytwvjpHAbA0zf759771FRjmbDqW5vTN3tNl3hxQl/ea7u/Zm3OBNu4f9gzuOiqp0nbbv/m8p5zzKuyLY1x8yYVI2x3DTJbaypq8Jve6VFpemfWsZVPe11NxVJ4mXOuCX+HzPRhG8PgjtxnE63DcA4M7H93f/8QT+MfPfRb7xqeENDHlZb5OwU5PzMgf2pgOju0IdeP0nTRRjNR9p6lpl6dsW+uxiBcy81bb94vnYwbTKm/q2aded6NOjTxiqZkPZJbnxskMujSG16LwhEp2HL5AUEn4dyR3w0IKcfNGp4VDDzsc1778Ik0IEYfAWQxtHIcNeJN7oHk3VpFx7Lw2+2zGx1tiHYnla7uCKdZJT389djTn8ILnPxedelvZUmOxDgJlPiXrjb+84PkZJlRvqYmeWvpLOSnO6Y5pdXHC/yR4v2M9hZQ6e8Xbr8bknnGR+VeMjarkyKDFplVbfkkiBunCNKNcNM1+4ZQot9i8GU8j5mf48aX8O6vaxBMOFLwewOHntPISpjRcW9YshWRqpeVljTfT6tunVWdz2YgXGrEDVhKXLUyKKG4jzGVw8bPOxAufdCJsAJ4Fe70MnD8TuIJIY+76Qpeyu57ah4tcZOks4+GfmXEkOOWcV2M8buOSSy9Wl+zE7n2qzJHZpC9qdU8rOF2WBW6ub8CGDysG8jELKdi9BTFqvnoi/2/Buy2QBnjde9+L6YlJ1BttteV2Qkb35JSRTsVBBqOYn19AqZRHu97UBAcxWVUAsRiAi0Vs3LTBEEMztQQnyJV3wEi3b8+CPbJNJHAVAARDIAxp1m3OjUYnyGotR/8+4PK+jhrPh+a24ZeqZq6+73237iVuS9Yjq0bxrle+EKP9JBwaC8i7pgNNe9ctuUaGLqPVW9NurOAYPb0ECsZHYQnHn3s5HlgYx2svv1xDlnZyXm2DzRd+MzlAxltnx67pFmnYs+i4CrbZrWdgOZay6p/WsVfwvQHRssZ7wQPXXP85PPjQw4hbxqAt9pUM3NCM+hhjK1eiVquqVZjATnNpSa1V9SUifSZ07ThXRyf6Z40PXviU3XIwxfuhpis3pbhcNUlpXcrJkHy9VarYR+bUwpENliNtmVJqhhtQLCF6mJobxY0oMbCIrNsYaSZALk1wxMlH4e2XPBMJ81ovfJ/f76fJPtbowQDE0LGClFHUjPcvSmRP+sshxtlwJU4454XYWp3Ei1/0fAl+z9YdaNVZOXRkDnLundnWWtBqGBnfSCeCqx3IJUw+g5C9DS7rkOvz6R0F37sjvL/v9a/ezPzyjtvxuS9/w7LTJEFf/6BAEuaM1Wodo2yhyqZi3HYaTTSX6IsLaDc5A4+948s0oS7o4Lhv9PMH+kx7Tw/BkprB4TBuSoVnk0p7e3y8sUwcO8VtBy2My2098GHgi6F/QtkI7XYJl4mme3AcyWUXnY3zTtwiq+ILJb1BXG+6p2v2cvV6wDF/T5aWmpn3eX2mshknPekCPLQ4gZc+7xIRR/bt2IW0nWoEqwJAFyAIqnYceW0gujONRjGkUabd+3xNyzAOo0y8h+T/O8FrZ/QM9vc3vGtiGld/7GNokM+dJOgfHNIN5Esl1JaaSvM42WpmchqDlT40qkuW57rOFAqeXz618IQLQp0+mjeTq080Abvac7cq5SY+9lokWROhaMZt90CP37wezu1uZpfOMeL2kbpZF2sX0+9oxrKhZr2vPmQjPvjaS01QnAbta/zO5HqLpXtydGsfzPXGAQdaUWsGseccXXcqNh5+Kn6382G84YorpNn7du1G2OHQZXYYWVTuhejxerOgoWb6UuNVYXCC1wAoR34xsGx5uNKf5fFeyH8meAVQKV7+9negsdRUF2uhVHInOXCEZoyBgSHBrgnZpBwQmMliaX5hGRNwJUW2QcvvyiVTUNY9Y4vEvWScd+1mZ+L9QtJskg7uLbsXJr/3gjzK9Z2Aeydg9UKdGhQgrGB5uD81nuwWfn6x5Kp7UQcnnnQs3vr8pyFhAEuouMubN+vXjd499O2kvHzfznKpIdQFgT7RC2Ks3fxUrDvkWPzbHf+J9//91UJMJ/ZMIMP5/4504S1ibwbmTbfGonhwxroQDFdx5p9TM2RlnaX5M8F7s3Wg4FVxSoFXvfNd6h1nixRBbqZz9DPs1SItScWWZlssXVbXmrVal51DhZF2OJ/LefDC792pE/74Ea6Zh0u94HtNqyyGI17sf2iApYP+iw0XfA4fsXdNsouC2XBh4IqnYBlvgMEqNy3rBmq7Zg09l8ObLr8Epx++1t7j8IflWMG1TrvY04J5l8FrQ7syc7cBw0f+/FuMw4+/GANjB+Mbt9yIT77rOmVDCzML6gTWejm+nA9Yl92FabH66RwobHgJXSLHprtBEY65a4qSLAd3+5khsTmWmyGW/5bic1//Fm659143FaMtrlkmzxw5oxnsNJXkp7MnnKldwBMZ2k2n4baQojVp5y0f9GP9ZHxI16Xrkbb/5lAkE6blrUyXvNb3+lrNv3flym6q5iZlmbl0ubnKrsuRtoKv0NURHKDE/J7CXrlyJT781iuQURVwmW/vJ2n6dTrQvNt9LWMBFoAsX4P0miNPuRylgWF89LtfxLev/4Lq8NXZqsUVztR3i1yyGm5su+M19Lo1tZ7J3xPSJtBlkT3nBHD+kCJ+H9X3Ct7vpt6gjxuVulptpXjLe9+thgIb/l9ANh9qxh13HevgnAUbtRqqH7Ma3G6Qg+5GjKo/3Z3M4HYhP88iV5q1XuybUzCXaWD+HjXT1VGfeMxIt1DjxqHZ/RsB06dy0pSeYr9lGGZ+fQrpFZQuzUWH1nDBOCWw4connHo8rnnxhSb2nqi+F9b97/L7XsFrI/QIngcRHfekVyLfN4D3f+Oz+P6XvoL6YhW1+bqUwbtf8fnUEk7XbVmO/8+ex9rSLO21vn/OxPGvMSjc4RqPPfzH/blWzkQtw3+2BqoMyc8neOW170Lc7KDW4I0lqPT1axIGT4KgeV+YnUfSbttkKJ2SEGkBPZZPky7SBf/ncHdNvhaH3wSvmXZuSrSgzq4sXErYZdosQ578DAIcytVpDTgqNJsTx603S/Edtt2mDBdc+nEhSiFdKZYLau3ONpuWNunNf/UiPO24TeikjAF8N+z+Gu03wn4Rv13VxTLELXyXTQfHnv1aZEtFvPOTH8BPv3ODMqOleTaX2nxc+3IVU5uNLlqV/u4yCV+UUXOGS/2ISfrfi1vAYhrP1fnfBN/VMHd+mvdb//CJT2DP1JR8PRejUCxr5CajevLp9uzcI+5Kq9HQOTcqtDgN87uXBRdj4jpSINMxtmARPOkhG0gj3YSpZY1f5ot30yEH3XrBy5wTruQGcaNWbJHoIhxh07mTLnjj0tRumCDNdBOtuufoNTE4Oop/uuYNqGTMTRyYvvln7NX85Y3gy7Q9pj6NcNLT/kYW6lNf+wL+5bOfQaNWQ7tu8/a94AlWeRTS8jKL6Ak7+9TWc+q8sBOljL5knopnL9i8V/B+d/aakO5iO43nv+fabbzlPe/TpEvWszmtqTzQJ23rHxjA3p27kXYiDdRv1xvIaEdyopnV5mlNBJa4yF34ucCpZbMuLXcVbvu558uf+uBOiuLDWqmV48eJ6pjfZ27PQoUGASjiNW2zcwNcW3NPV6tcjidhmC7p9dZfZ1VCC/5iHH/8Ubju5RcjzbigqtsHv0xqOdDk27+XBU/6uTZJ3MbJ578RnUwGV13zd7j5t7/B4gzZzHbGzeWXno+DRytYu3Ytthx+sjSf+AnHovArk7cDDLiOkZo3OqJ38/iS6mIVu3btxPjUtNZgdMWIxrsHjz5065+ZehmVnsHCvaaeP9Mkv+Kad0h41PhOJ0D/8KBQqpGRFRjfvU+CZ3GmVeOZZ4ZW+QYGCp5+U8CJS1XsnDTDnHvNI9l/vRG9F7/OaaPA09jGnrkqneBLsW6tVu+jenseG0fSi5z5wMtyca/BDvVzgRWbQvjF2IQ+ts5zdAb68YaXXIInH7vR4fcuqncuwt9nr8n/7wTvLdqJ571eJK7LX/ty7N69ExM7d+tcnA/+w1+jsTSuruX+8iBOOvlctOheOA3bATtqi3R1CmIZhgoukzbM+jlfryyXnTQHCt5H0YEt3oEab4fsxPi7D38M+2bm1KPNHJzjVGTys1nMzM6onMlyIjWe5XCBIq4Y4mqpsgJ21lsGhaLNZ9UZKgfUwL22q+/cgSbGqzNwg0ebLAekPZOhHWDRfWgXqBhGYOe8+SKP105P+jBugINhXVRurdNWziV5k6dPXn/t6zRShfN57b7deXvupn1N35t/g2z5xSPI3FSNNMAZF1yJJhJc8BcXolpbxPzEFJ739NNw7ilHKzvZu3cv2u0ETzvvL2y0W4YFsZY1RSqEtuYILU8P/iHShYO4FfASgeD3/03w+2m94FPpu4KSG/90L7763e+KK+fPNB0cGsYS83Z+eMeIGA1W55x5p6n3QZa5E+ukocayuyTmQAP23HVbq5fNpu+y8ILndcjtY0DpgzSZbwEX1o/HyFb5rzv7zaXConJzg7ISyE3D9/cya/wm8FG+ByIMjLHNEDV5wEEbp55wNN7xmud13ZQ/dsz34nvBd69Jp6TYhtVIA384NvbsZ70ZDXRw3nOfqfR3bnwSV73kAjVu0Idzrs2WLUfisCNONndDy8Jj3kQbk7S1bgKyZLKZvtHF+U3hu3pdJuAF3+vfe4M6X8mSeXQRqRinaYqXvfOdVp1rW55bKQ8Y9ZcTSjkgoVnXMIBC1qL9ZsOgXp9XMxU08gT71SC3wQKy9c7v3z3bTWV08C6DthBhjhg1I1gKuqPhTdQ4agg/Y+P6Q/T7J3bv0nc+QYFM4E4kgKRUKVvzB+/XUbcs6nbDC103Tm8qJmBJPspGnw8OD+Dav30lDls5pJGsjPIP9O0y94Ejk9AySPDGG6DP56HHZz3z9SCP6annPRWduIVocQEvOf9EFDJZNHiKRpzg0r94EZJMCXc99ATufPBe3PfEds0XaqlBdRlml3vTBDHWsK313GIcp/H8+ZEH/7AfEaPrTx2I0xW88416KLczrv70P2Pv7nHU1QiRiK9e4kmPBGg4cG9xHs1qTa1XFHK9VlVaVGBHiqNQ+SmWjI2I+ok73jMU2PPIfV+ZzFo2QKWYRV9fCUdsWounPOVMnHXqUZpLx5YvBWX8X8+YEl7zZzffieu//WNN6uJCsAlSvt2Z5WV83R5wWfPN9xuubwJM3TGqTBU3btmCj7z5cimdhhj3VO+6m8ALvksv94pEjU9x1oWvx2IS4YKLL8D87BQKnQinbFyFUilEK83h4aklVJsctJxBJ43sEAWlecQ+HATuXZvj01tKu4xzCDQLHHT7yAMH5PE96JaChG7o5wbEdcsnwHd++TP85Le/F1onDh1CTa6iH6HpnJ2e0lwZGh+mEJx/y9/zNTTBbe1U46bSzDdaNVWjSOvK02wHGR1Pyu5RNimefczBuOaNL0auWEa22G8bZL9wX2Fo128vM1qXq3V8psvecDWaHfo6etrlnOrLdQAAIABJREFUUyVoxs0aeaH7s++6oY6GBSt9SvxxqHRRCS574bPwgrNP0LHf+wvebWSX71NYxuJxfYc8H69TwbnPfAlum9qFv3rBJToAapAzfJMY2VUrdVgz14vsZimmKw9zvT1NWemby90Va4Dzh/O2Pjxjhz/buA7boA/ff+v+ZdmeAwB6BW94ke0C3TiAxyfGcd2nPt2tvtHskHdXLvcp6FuqLii4o49XvskTpjsWCFr0buNLKBa6DPo6FWs6ETauGcKpRx+FVZkW+ioZTcV68gXnoNTXr5mwYaGvSy1aFsufC94s2DK/3FLDBB/90vdxy+13q7ikESqOmOhNvQWLPqOwdNQqeNZBq0O1dW073rRvbAj/es2bNQv4QMHrda4L2QteZVKXiTQ6/XjqBZdhW20ef/mi56BVb2LLyjE8OrFP1TVyA3RapROumLLi6RlY1T1hROtMZI4HkCyPPekOqGQzhevuleC1XC5a9qdGdjnc3VV1gu+ZlUYm2LWf/5waLSi4Rt3OSunvH5QF0OTLZktNlS7YVGBF/63+OlKtoibWjo1gKBfgyU86Fcds2YSoVdcD7dqxC7XxvTa8MJvBEccfiU2bNyIln8zNxe2mTeLjOwxeW9ohjTpE0U2B8IvvovrPff9G/Ow3v9dG8C7OZgAZ1cprfm/MY0pj7dR+8BCZxwxKTzzpaFz7+svUb2iwrxVgzD0ai4auwCqCdm6u4vvsKpz5lOdgMm7iac94Cvt8sFSr2rkBpYIILzygkCCZGkRczq5Yh/UIxT3ugV3NPpfJWYDrqWou9uJhN9qu/5PgvU9d1qYe8KHH/33qhhtw59332KSodltBUqWfB+GWMD0xhYQDfHnkB4mYmVCb45gth+JVL70Mmw9ejdt+eyNKGaAl2lVq57W1Wf1b0oOPrBhFpZDF/Ow8CuUsTjnhKE3PDDlwWX2qjnPnTpdga7NFuAFml+rYPTGDJ3btwa6du/H4jr1a/MgJNYMQe+d4+JHx69XoofEtHk9YVohebIGLHDUtoGUBhCAWZVmq5PHuv/1rbDhoTFC1xQn+9Gsz+ewgVgbhLAp/Vxk7AkcfdxYerc7geZdchAyVqNUSNsIDhIsDA8gXy1izdr1AnJGVI1ixYrR7uBKHJmkABYmjUUcnWEQ80pTdSY4E09DcnQABEUhO5/CC7+5q59QP6JZ2Zn65YGBPFePGu+7B17//fXWnkBUqfD6bU8co/dLsvgkcdtBKXPv2v0eZGscFcQ2PRPTuuPVmhARIskTAlufMeoKCtKbTckeXt3Dc8UcjIjBT6dO8WBFn2XHSbOBHN96E2+5/RFOz5xc4vIEjWW0fdNpskDDNZuuxPUkWHNPKgMdAneWDE4Q0us1ghxQ57pqbasXOVf7dmK02pqUV1TE0PICvvu9q66qVK3DBoOPiJW76tbFmLfXadPRTMbZ6C+6c3o1XvPRFiBZr0vCxdWtw/AnH45o3vQOtbAGLSRNtXoeHKDLOIOdQQE5TgheLiC4kxz5CK+ho1Bt7DgXKaWqwgu//UfDLhYHl+vay1V8G++ZadXz4X76IfRMz6g8XQ4XDQfI20+bT11yDdSvYnWrvtvzdH/CT4t67b0UhZKQKneaktIqATj4vTIAFHg76L+RCVPpL2LD5YLTSAm689R48uGsvanEbDRI7NayYAmCDpAmEEueu9314nnZERJGLwaEMPJ2Kx4ISG9XwX1f77hZ12AnLmX3uqBYej8b3b39sG2rzi7bAAa/VUimUtfvXvfQv8Mwnn2LxkGsIUUbAymPkOABdMmmKE858Psr9Y3ikMY0rXnwZpsbHsXHzFnzn+i9isDyAxRCYojYrM2B3bIp21EQh5LFsAZpRE40kknvlBGveY7vdtJZwztbNZTVFVKd1c6Q6Q46H7vvDfsGdL10uI077C16+xEnRV6T/8StfxgMPPGoYfKOpAf2CU8MQ737Da3DcxoN79oyVZ81iJLj/3tt12jE5Y9wbGvTnqE9qiswVcffObdg6OYcmkS4e40VtijqIOHyJ6ZXNf3CsXetatSKFaWmxwDHqqYQnxorr+KG14EZbaiyKPqaqHUu+hbyOXtFcHfbQpQl02CCPAUkTneTU3z+EQqmgMXC8xvzUAh668x489tBD6Bvsx1fe93eu/85Gu+hxCbeIim7m3yqgIU4+66XIlSq4c3o7XvXyy9FXqOCmG36CTjaDe2tTmFiYwkJ1CUnU1LNVin06P2igUtZz54KcKQAPbK5VUa0t6dACYhWe/MKAUCdq8339Ayb4/YKXIOmJWLVnl928+6k3g+IDfOTrX8KOfVNYYhM/o/OGjfwuVUpIW21886PvWw4endYbVSrFI/ffaV2jYYDhwiCWwggP7d6N+3ftA6e9WD5uQ5DIfy+VCAtnNJmKJj5fsgHLImW6IUd8vU6iEiOVymzRr6ZDaDqIjUenQDz/j/dLS6Hed3fsyMLCnH6m1WAA55s0+R4e1yZ2TmQmv6/cZ0WifF6t2SPFPE47chPWFAjqOJaP8n8P2bq9n6Z40jlXIFcawKONaVx26aX49fd+gioifPeeW7Bv9x4020ZWpZvUHB1X32DbOT9P5wNx+geha83+56idpmYOCH3V8CgrK9OtqavIC753Vy6nKlbrPfBrP1oRgEen9uKr3/sBduzYY5F1DC1UpVREI47w7fdfi4JGoi9/+c979IE/ycT+6qGHMKHZM/TpHbFMleY5/0QjQ65dsdBnlOwMO3nKBssqYjWfyvr7gU0P2YxtDsKzur6iXYNzaX2kyc70coPZWbBkFBV0BIv8uwNFOFmDMDXblnTEaLVuWLhmJLlBDBqz2gKZBfTJlXweh60exbFrVqLAw/6kOZbOMoA97vRLMTK2FvfM7MSHrrsO1/3j+/GlX/0YtWZDKHwjsvI3mU1SRTe7lm3q/L2OSHcDE2z2OQcgG3pJ39/f168z6Q2Asna2ZcH7kqXPT33x/8+jvP1KpMKtA+CaT38Ke3btpeHRTbTqdRtRlglx1MEH4QNXXWlND1phnuGQw9bJCXzlxp+iqeF/Hevf1rFlxqnTgmesLas6vyDghydcqFhCwZfLNoudqKF65G2gAdeVAmabcRe75sGDPNpEwjZrQ76g+eHlXj3l+SFkJvmz74ilC+Ln8h54f7wWByl3hxvFdlIlf6fqFzLa/DwpQlF8QgIErVAWmw8aw6lrV2GIz1EM0LfqRJxw8tn4rx33497f3or8oavQzmawZ99eo7g166jyUEhWNDXg0CZue1STsuY9ERX1ZW9aAI6Cp1vSc/oBlAzAKfyuqfeIneOieTLhfrNJnML65gCvv2EnxTv/9bOYX1jA7CzPRcloECJbq3gWXV9fP77y3ncgdLXoWpDBh7/2VdQ4NiUb6oiQYp6dtBS0+T0yham97FtX0NbuoJ9DgrKmvS3Oi1NbtO1gTXB2x4F6mhf9Hx9SftpNxTTiAidulG0sunwfq3vmq42Ry7P1LD6Ym511J1waLz+roo65EgqFFoAADg/3NdNvk78ZTXOEO6d1G1hlYA/LKszzmYszRz9qzTqcccTxeMa5z8Efdj+EY9cdii/9/scKPHfuG5eb4eeIE9COxGWk4EV2FW3dOo/ov2klaUH4HDq/p5BDP1FOziEin4BuK3KnZfYKXubCC77Ht/cGdDJSPTVzL/x//+1NuPnuO7F376QO/SHPnmANtY+jxZ9x+ql4yYXn4+a778FP7r5LTY8WgNnid32tZ+BqegPPb8/qYfg1Nz+HFStW6Pw5G49mw5asvNvRYpG5qwEA7nwZ1eXdDHrz3bQgoYY38ShuGzHuJli6oNAPHKBPlabHHeXMS9Vqd3gSNwCFwvIsn4MFG97nAlubq1U7FoSVNzfixRNMbWRMoHHnNKp8xv7KIC48/VyklTwuOP0sfPOOG/HE9m1CKcW2nZ1HvVF3/YghWi2jsrE3kW5LVDNOJGvUVSuxCdaWnjZ9+uh6+voqA0a+3E/wPbTh/yuo289fU1vCEFd/4iNYWKhpGjUVkBOyeAulgQEcvPFgXHjaSfjp7XeI8EfByyfnKNiiLkchtohLZ0JVzTS/3REofSbAYI+WwOY4WRrlhwaYZtu5NLxml11K4Wv+KwVIjbWAVZ29jrTou2jNh7puWneqhI/CuxbB8d1keplpMDPgKRsayWra1p3ooTMAjEfohyiYh7comxuBFUaCUayzX/6Cv8SetIaZ+TnxG7Zu3ar8XE0scYLq3LxNv2KwFxEws1OuRGyRGyNPYXkursrD6mewdjVuECrGsuD/jDpki9OFcntKH12hH3CI3ds/+0k0GhGmpucVPTZqNtRIc2Q3HaJhwjR/vDGdZknBMmcv8EhR81MUCjXMTmCsKHCisBgQSUhu5IiaHbN8COIFLX2n2aW7oK/lG1ivl58OQplgnbjhzJ4f70n3wSDJV+Z4v0pFdUJH3tqomVE4lyKAhNTuXM4CLlLIXYaijdeBzDADRDJ2+Dn8PSNsfbabK8DTJ7wbsvGwsY5Uo5AGDlqJJ537FGzfuk2pGcvNtCzjeyeQNFpoVGvabETl+Kw8a0mhk07T4vApy9U968jGwtrBg1AtweXxCmj8cVVdyrCDGLuTMRzdYZmdIF/TuzE+8fWvYNvEBKrVprB7Tmmy82dC9K8YxvCYnaXOPFrRdKXs8GRrCOC1Cjx1SVagoKofTaHamkJju1aKRQmRm4BmmMGUmgl0Ph5HtFD4oSJdHlIoQTnrQAvgF0QWhgER74dkkBxHtFkwyCyDGtls8v1sTc7oc9hDoPo5aeWlopWRHW9QAx8IALmxo1xs/seBDxQar6l5QI48yvunm2H0L1eSy8taaAN0Yqw6ZB2m5+ew9uB1WGpaUBrX21iam0dSb2tsvHx+HOu93IA2JdQsmT/3zub4s0GEOAnn+TuuwYP3/j61xTlghu2BPt6pucesZQ16ulb473sefwxf/vH31DI9OTGHQr6o1Ee48+AAVh98sB1Nmg3VDcoGDGq0zLNj4vB1FDoXRvmyNCpAlnVoQqSOOSvf6o48UWzSPQrMDiCgNjJgZDWQfycSSC1TuYSU8EpFAxa0UI4M4vv7/WYmMEQLQjfB82vM1Gd1xKgd48n4wE6I4t8NCzALofiGpedm0xpINIPVrAFfTyvjLSqxczWNJrZxma61kxiHHnOEaF08XbJEhm0mr3N2o0ZLhwtatZAwuKdpG+1a13Xt0lZwshGwJjNXabz/7t9Zde4AjfcVq16N9ibeC/9AwXOo39s+8SE0mxEWF8m1ywp21TSMXBajBx2E0dFRTM1OyXxT+NTu4eFhV+hIBXuWSzbtsdJX0QBFLThLkO7kDC8gj35ZfMB0y7c5G8uFAxm8hov5oxOiLGswHpoFexFTsB5yKV/L+6vWaoKhFQsw/qDbopVgOhVzWBOjbaNPSQDq+TOmLgtWtAIUsqhSOm/Oavn6HV2PQxap8Uz1CELxWjOTU+gbHtIZczT9tbkFJM0I84uLQv40ccMxj72LcmLt1hv8rF/rVvIbgefsulnB9931X5pzR43vFayn/nZ/2fPDMqazHAf4zfC2f/4Y6jXOrKPW0RTxBApCjQkqgwMYW7VSJowaNzDQj3KlpIhVJyGHduKjR/WGhgal+eaKLKf2zQKeI0cky1MmqWl2HLdZCk260vwkoiuWHtq1fHRv8YGVNN0UrU6Mpbrl8JoL70AeDwFzc/HavE9/eII0iqddOl9NzNxo2NY7wOfz2D/vheZd13Puocv3Szgh0/n+OMYSz5yhu8uRjt5Gp2F8Bs3+cz32XHc9k6/xusppnLBAQ9DGjZ3pys8Njrr3Tzd3Bd+bpv1fgveVp672uw/+xNe/im3je9FuJViYZ4pT1BgzPiyPHx0ZW4EWz1UNM+Kr0ReroNOJugQNLqhP88zk53XiIjeLD4i48GZuE12b16FGWquz5eMKLFmo0Gxao3Ornq2UyooXFA4hT9LH5LPJSyfzRXPeeVaeTZ82KNfq3/LVDgWTmddxIxaUskjDz5J7IP2cfATm7AUSSjtyORQmT6xmcEaloPnX3D926XJjRG1Zvdm5eRFccwULUvkZjG98u7lMfc9Erl4l9WCZZh264FOm3R2lEtx3501/jsk6qEGvO+Dsdf27p8nwwL/fct+f8L1f/grNRlvCTHQSFGfR1+RnVq5eheHhEdGFS5Ui+ocGFeRRmymkpXpdUCwBlmqVg48NauTf+BrCrjqpmUOVNJ3aOPq95t80gEMMbCqXMSoM6vRQrVqdecx52w4r5rU85GuZQYQGMXIaAyJ7boQqwR9r6ba5fPzZ+2w+o9c+Rur8PWuVokS56ZtKK4k3MHhsNPRMrD5SOAzWuGGZxtWjJtrVpgpdeY0zIx7h5v8fkE15gft2NNERPMXKtZmL2+i+ZAn+J8FbU9//LvgDTQzR3XaY4m0f/QjaLaZACRYXaoJZmWpRUwZHhvXf+Pi4dn+pr4SRlWMStARcLGjB+DN/x8XwttyEb5G3bwsiBs28lILSyVGJ+V47KcOdwuQHIzmki8+loNH7Sofbe3/pDyrQcARC0pEBONwYLHeaqY9ccOioVu6wQglQgRpLp20dHMQgtMh6gMiFlvdzTDsF7wEm4QFRpBm+5CJG1RrWj41hvLooZJM8em5A9e/tJ0TDOnRWgM4vW+4eNsKHa6QgZtAF51IE997xn1aW9RvCHxLYE+Xv5+cFCu2/KbzPd7w+XP1PHxNyR3Ig/X3o2oxo+mmSy30VbQI+RK6YR2WoH6NjY1Ys6aKCnIJdslTLmUlh9K7rlg/P3zP9k5+LLWgSvu9MGzWLx6eyscOKIkaNtrZmi/7FPA1tdoyCMoEthuVz09Gy8JHVu8+TJxrN5dxex4rbgctadDcPT2NgOQeIm4NTudsRSoWi3BTNuoE+BiX7moHO8AlYX8igWmvg3GOOx9bHHkGLlb/hUUxWF9BkZuHaprgpmSlYCuomePAZVX20MSuaKJY4i6nYwUrYstJe8N1u1P9D8JYO7F+qPbCO8++33Iwbf3eLmB6cwVpvttRMuUTggSzb4WFpACtffYMDyBazGBoelpA0BsydskBSJk210jidHr188iMbH0mioKnnmTpK2RxWrTyWgosiuQsiiL5TlwvF8WFWvDEXwE0gi9ED7XKz80RMjVmlptPXu0FNis79MaQy5cu8dS2uAB/bZEL15hYUh2iKSKGoZ6LF8CdcEtvn9TIF+vkYm9eMYSxbxrZdu6U8737b2/CO970fLUcKFQGTpedSHpe/+FLsG9+nieIkYDTbCRaqDdQ7MaqLiwbwaPCT9fzbKBEneEvnTK99D1ovAbFX4/k6f0Cu9+8HCp6HF73tIx9EQ1BigrbTiqjVUV5PXj2FTAtAXln/cJ+IGMLdXQ+4hv0zHaLQchbNKzjiyRAO4aMrkOnvOe+eu52WhP6W9Wqhda58aahcRr/XEaU8Lk3om1kw/T3DyZvU5Mjyap2k6Q4Tcpi+LI8zb0a/srly1GZtnhangwxi5042ctiMAB99cxPpYAaetunm5pn1KiCfy+Ctf/VaHH/EGlz7/z6I6blFNYf84js34PmXX4HxxUWlnzwHgHLaeMgqvPkNV1j/gPy6I7XyKIG2O0/HWciY6SspaHrUAMG9t/0qVSDUtfUuRXP+vSfH685e9b7/QMH7rIAb4+d/+D1+cvNvEUWphh00G0SnClocbjyadZqrQl8RpQFjklCQtBIM3vh3wrvM8ZmG+d8pv9cJGHbwMXc19yyHJnJDETvQfdCMavKGQZTyvZq358azuZRMGAPsaFW6CnXwdlujWfHj2H07811CdHiBdx3i2jEbaJpm0XJUFxbtaBN37h7TNm4QnW1HbN5lE9xkwgYyWYxWivjsR9+PsFNHOw7wzre/B03Xa/jlz3waL3nNlWh3mE1YZsHPf8HzzsUZZ5ze03NvG2B54ANPgmSvH/sarC5BjZflvOePFLztIPtyw/APTODdMZm9Qtfe2a/pwjj3PId23/g4PvGd7+pExHbckuAzjvLL06ZKRUP1hsaGke8rOnDFJmPzxpka0ZTTRZDRQj/JtI9HinNx5+dnBaHq9GWNPOF4VAI9OSFryvmzLO8yFfIgi82zITQqGNMFYvRc3ADcVLQAOvzXCZpuh75eR5u61Mn/TTUBx6admZ7pNjsYNsSAyyJ6uQimkJrQGQu4oiWjpVLzZbkfV5x/Fs6++BkIkizGJ/bhwx/6FBqMUfJ5vPTi5+Az//YdTdu01JDQc4APf+BqHd7EjmGnx12peSU0hWZgZ6VkUdoJtd/1+/9Ig2yha+o9r/5Auavo3zPHpTeN86aef6/Xq7pxfsjMUgOf/eEPVEsnlEmTT1x5lpMeuLitNjYduQUxazOu24MPRvNMn7V61SqlQdZTl2JgcEAIILVJp11ns1Z3dnwyXkSMWB5w3NVuRvochpix4z1d5G8Rrx18SOaFnbbp/L3O77RN7eff2IGExmSlv6fAVZRhwFZj14vx5ClwKYeCNxZebB4A/y03ALqrorQ8aEXIxsDo8BCe/8wzcfYzztPnXv+5L+G+ex9WF8xJxx+HxflF3PfYE66WwbMA2FxBwb9dNQwDgNxhB85S+yhMrogNopyOqfpEwXoO7rzphympyl00rqeTpjdt6BX8gZvCd4dw0hU1MQjtSBKal0/827cwtchTlFM0eVhRjuYt0YwXYs4Do0PYfMzhOqyI5lY+OZNRNWtsbMxKmSREzMyocEJzPjQ4iGLZXIUQOmnB/1fXm4DXfVbnvmtrS1vS1jxbnk0SOwOQwKEUuKec9gKnvbSXnsDtgdIUCJlnZ3A8xU7ixHYcGw+Z54lACCWkgRAgKVOB3lKmACEOGZx4HiRrnqWtfZ/fu761pdLnKk8e29LW3v////u+NbzrXe9C7stROh91Op7akJ1nLyRufEK/EykURSYVaURXnpFb8TTVo3zNmmCxEzAD7Ispl0zrrC7bkr0UvW7a0UK+IDgmsIbrYx481cLJoVHNigXIaW1stL/7vz5g7/3QX+geb7h+kx3vHlDf28qrr7aHHnzU3jx8xOlgVVXeJVyWsS2bV880Y85C7sTO+aPxa6E9MB0Azn+88LViZUN9iRY1G7HTwiew4D9tgj9e+cK0jYwO2ugINelxEf1cLqzCKusb7Ma77rGRsYIvvAK4aeuht34YgGTalp5xmoIh0Z1SHqqyLHRgTnN5ue19Y4+iZ1JBkDayALILXACBovrsRSzk9PrJ5k/eh0UQ2WIKfzzuQzAEAVeImSq/m8gbs0UXtVlIocYnrKWp2V7ZvVufB/jC6zWpuTTOnM3lAZUC1ERGrhD6Q3iXtYs/+yn78/f/iZ1z3lU2ylBirFxFhc1ra7G//av/0973Fx/Q765ccYMNDY1YRVW53XfHbXbeZVfa0PC4VWRJbSutOldtJ5+yxD591pkl9ywnrTx9RrHbvzczrox/w2FUeZuFr6irNQTw3E/8UZVuloz4fzH/kgKdtqGhfhvo7xHPjxMERCqQhViiaLbveJ89/Mx3bISceBoR43IbGhq1wd4BASInnn6KbxLkT5P6BOkPp5vFZNwZlGA4dt7hWnDWa6qzK3VT/bxCD9JFk7xQwmvUyiWSoSNaIHikaSq2AMeGzm7i2zvxwjti8bGHDx6SLw5M3a2fa8fOPumeGkZ5jFSuYOUVVXbRP37CPvahP7OxiTErL5bbhZessr7hwVJ9YF5Ls33yzI/a6e97l+bW3rr5DkG5bXPabOXyK+zK1dfZ1DT0NLIbh68/9ekzbemyJQmjjyFFDmyJZJkImRGTKRZTvJEKPL/8wVPFLHZfKdLMFzcwG579r7Ges1X7+o7bYH+fHkplzjFx57MnHRp2fzZjX//Bv9mLr79pY1PTIhYAWHQf6xad6MTTTlYO63VkR76Ae0XWmPaBQSwmChQUPKj4IaoEDWtyKs1uhWyQkCtRq9Vc4eVZOPgEU4Jkqd2X/LMDO0Q+QtuS/JlX2aZtoLfX5+6Me8SuOCBlDWqc1Ewel0VNp0YPlrEs+N6Vl11s/8cZp2mEKcdb6Np0mV142TXWOzis3ye1nN/eah//xF/bO05/p3372y/Yt771gjbF5ZddKM7ffQ89rnurylVZZXpOGzauKrVuz14b71FMGH6pVO3Bu+TZo9bw6399ugi6U54oxrFDSsWXPwJrwnxwUnqPd1tvbxf9jG7yknBh7K5Ib8SRs6Ld9rVvWtfggE1OeH38eNdxGx0ascVLT7BslUt0ccpFhkgsGnrU5CpFnypo2iVpFyYPd1JV7SPNggZFCkX0r0pdRc5pT4gsTnoBRpG5pmI6HKsKmrphnLbE7/Ue7ylV8XwGruvc6jDHeLGEoP2xKW1rqLV7d+2Q8jUz4tHpY2hh7A0sziWXr7KB4RFt3urKSmtvbbKPf/yjtuzUU2zTplutu3tAz2DjxnX2nef+xb79wve9M9bKpAmAZbxhw7ViA8emi8XWus2ur6TFn12QUVT/mx8/W8RsVtbVKZUKzvz/38ILiJiatKPHDtrxrmMOqGRhq4xbQ0OdR76iKGdUYXLyAtQp2LRlduODjwsRm6bXbmJK7wG/bu7bFjijNlPmkxdzHs0L8k1Yusw2hY8xoN5Kfb+6psZPU6RsjAdPzRK4GRZN8irqn/NNhO93yNZzfRDCgwcPeaahnzlHLZqrQwtIFbIUs0mnz/XX5RLmtLfZI7t2WFkmFW2o7lERTGij3KgqekW7YvkK6x+gszhj+YpKa21ttE984n/Zyacus3XrblR9o6q6zG7eeKNtu/V2e/XNvUpr2bCtrc1WXpGxdetXKo2L9Yrhi1E/iawrFrw0MQPYmcD3Nz95tshfsvnqmVGUs4oAsxUewhocPLDXBgd7rRZeO4CLUgLUJp3gr6JBSnV4qAzrpazJDp/IVtj6ux+08XEXIOrp6rburi72bhpGAAAgAElEQVQ75R2nWi5fJVpWTIuWdEcmK5WpoBITsU6NjothorKsumYq1FnDahJjSAOHiD0hhsQhWqRUL1eRZXLCTl12sv3+dy/p+zBo8dke3KWWyoT5RwnWT1XS403ZwalvW2wb1q6yGvAHZt8orYJXMCZ9v/8SBxeKduXVq6y/f0TpcS6btY62Vvvfn/yELT5hia1be4Ng7o//Px+z//7f/9SuX7fZDnV1C/cA76+rr7X/9t9Ot7/+m//pZUNflFKNI1SqWWjJzKT0TsLb9CUmjoIWXpEqIkJqNPgjiYlQdhbiNWl73nzd8hUAAVM6QbW1TIScLFXUWCzMLQ8eU6uHKdpUQWaNhzc2VbRVdz8iXzvQP2DDA4MKZIBvS0UWsPKJcUX2oH20PQnmRA8Gf54ia95P/w5lZvXDe4Qr3ZuE2omQmS3X3Ly+48fVri3oGWsSfjHQykRsEOkyNWzoz1Te5Tc+eebH7NOf+JiVic8fEqN+qpW3o10z2F9iNpWCQCvaimuusy4NcCK9q7B58+fY587+jO154y372teeUoFn545bRL9esXK9DQyOKACtq6nS2Jfzzj/b5syZ4zUTLdfMBogTrhOffhLiNbGh9TMWXgUH8B3pw/6RyH+KfNlBv3/pRWtpbVSwg4hIZUWVFgUkiTcLnhxBhEqjqp5VauFFa05pVKE4YdduvNsK9XWS7oSQSLfI0tNOSRRh5qP5o4oqXq7CdXNQfFQzQUrB4kaD9IirCN9NLd+LKR5TkB3wRZzgNKqssgmdBsq0iaemVm91nrjlkD0rFq2hps5uXLfWTjnxBCtOjNjE6JBNF9OoD6EiaeEpKKmBdEjmPsy8HnwmY2vW3mgHDxyVqa+qyFnHnFY755yz7Stf+arteeNNETm33rpBa3HJZVfbRKGo3L+utloLf926Vcm3J1WwpK9TMu+zOIhR7ZRf5z+58wzI3bNF/Bw0qap8zQwpD3CCFl8gycKk/fxnP7Y6nW5Mablm0kRtOJgutAHzoNVpGukDTQnw4NOAez3MwqRduXqrldXUWqEmp46b0aFRW3jCPB/Gm6pPXjIlGnWFKZogRGAYGxcaqNl3IVGCWeUI0cQwNq7UjxPeP9Dv7ohWbIE1nutrkzKIIE3OUPqTpETGoSinqdMANR9835/amiuvtPKi2ah634gbmLfjA5SC2RMBltDHXKWNDg1IRzdcJDgF6eimzV+wPa/vLZWYO+e027nnnmO7du6yvoERe9/732Wf+ew/2NDAiF199RoJOWBl6eVrbKy19etWWyEdDA9WnV41m41DZ66upyQL7ylfVCW18DwsdGkrq/PqWg2TwALRqPevP3zB5s1p18PioSslKjI9sqYEYPBv0LMQHyZ6la4MHHSkRRPY4cWNgl25ZqsNDY7ZZFJT/qu//JDt3vOGjQGkZKkbx8hxCi4geUNC0UT2EE3Z+XlAoZxexpqqmRLqUlKB4JRE+TR2vrc3BZ07DQtOOS9WT8BMgXbirJ115sftr//yz60yBAJxIakEy3Pxh+sNlVrcVOjigQPYTIwjYDaDi0RN5LZd99qvf/Vb/QYWcV7nHDv/gvNs88bNNjw2affct0uiDj/50U/t4UeeUNBLCkxgh4u9Yf0am549blWAES4v9QSIfTNLVj3a2tN8HFkGsHr+AnyKOSwkCQlFvoUJ+97zz9mC+XNLrUPUkTkdBG38Hg/K25jSlIbkU928uYq0s2UyOoFu7op2+bWbbHQUwWL3ids3X2vNjY32Vtcxu/OpbynIms4SKnncgUw65n1oYKjkNnhw1No5wQgmkwpiobzWjXIkMLzntJ4ZzPhgXTPbSySGgk1PeD0cw/+h95xhl1580cwpUtk+gTZJf4aYQSdM/p0W7TQYSBOoIVKaDfb3ei1cQaHzCCnFPvTQl+0nP/2Zfrc6l7M5nW32sb/9qN1//6M2VZi0u+7eqef58EOP249/8gvLVVWoXeqEE5fYqacttb/6q494FlOqqDocoRi7VF53/19q2UoFptikmV/99FktfCg1lFUjLwKJYdx+8MIL9rYl80oX7sAIxREP1hzzpuqWFpRJjZU0BjjJMVIfZ8b61CQPmKbsipWbbWh4TH6Mn9+983qr1M8mbaJQbhseecSmilkrpJ1LkYeawMjQqDN3ktwqAaLy81SM8I5ZFzwQ8yY0bpPbIOAsFZhgoKZIHez702eeaZ/827+xbMYBHW3eWXNrg7vnTYre8oQLCVPuuZUTPMrLM5rS4dCtT5f2RSmzJ77ydXv+hR/q3/nKKmtorLWLLj7brr9hs7W3t9qKa5dbTU2t7dh+u/3htf0im1SUZWzBwnl24UXnys/roCVwYAY2jgifR12wF1980d71rneVXIBboqQfHAuPaNAogVoNufekff/57+gimhpqZ/htSXXaETAvd0bO7IvvBZAwO5xULyrgGjwAVTm0vNwuu+Ym0Ydj4W/ftlYkTtiuba2tiop3fPmf7EAv4gRaAu3eqfEp61HBxrn0sF2EUSeeuQKxSCeT4qNOoEy8/8y7TxBKKLdcJmNn/93H7S//x59bVZXz54Xvp8jeEb0Z90c2EbFCtGPF5lIRKfUE4ttHhocS3Suwe8fSv/P8D+3Jrz5dGsXe3tZqly0/Rw0mdO+wyeEu7Npxjx093qvnVYuSRUOtrb3u2pIiJsGoW9YY5SJH6qQP/kucwzj1EeknU/+sOmlYNAYHEUA9/fRTdvLJJ+qGCXLYcW6yEidb0bJDnDxQmbBZYzuFf6dxozHvPRZDQVW2wi5cfr0NDbvCJH7ujm3rhANUotGiuyGarrSf/eFl+9Lz38O5+jUUnWHTfeyYn6BUD4/F8YDQF1dky5ioHLku+IKZzW9pspvWrLD2+nrvLk26PCI6pA5dPcA0GCk2gOP4bvaDCqZzLDVtmh99mANZiluWJJU+i7j6rz/9ud13/yMKRCGcNNbX2YpVl1p1dXQQZ8VfuG7NRhseG9ZmbKqrs6rqClu95pq0FgCSKY1TQhGMx1my6SVqmd8Hr9GhpUnzVz/9pky92o6GR+0H33vBFi5aIOozJru+Nu+88SLFjBk834WC3SRi1nkgihjl99ko3sHhgVROKZiozsCvmaxdsXJTCthM379n140qENH/Hu9DuZQHN5HJ2LV33O8AROo2IVXr6+3zjtxEeIgALiJcFt55Zj6bDbPN6Xpww3orKxu3wnSZGD+FIqVTb2TgofC8iBf4S2QE/AnCCWLnnD6PH/izpImfNOZgzzJwwQcl+eKE/Dob9Pe799jNm7eKOs4haG5usFWrL1fU7uaYg2V21fLrQEv0LNubm62uIW9nn/0PrgyKi0nxS3AHFUeAxaSNHHN3JLUOd5/ANU3+yPzyJ98octqBQr/1jaftnW8/Tdx1ghcWlO+HooKCiRTQOfFgZgge9fN5nXOVdsUpd7NeUSJMRmcKC3Xt2lu18Fw8alcP3rlRHHTyScAKoU78fuqfw7Uc7h22TffdZ4VMJbwTmxgfs5HjA15jV+UpzVwTugbxg66TolVDy8rmbH5tld26eb3oymEVwjopABRVimmODkBxjqJZg00nV5WYupoNk1IltzJZUchp1BSSmBpK/1OKpdebdR/rtWvW3KgaAYgc+fkN66+xyrx3DWsDT2ftokuvVhNmLpe1zvZWe/s7ltlf/MWf6RoEa6eqYty74whpzFnqsIkMzWv0qbmCLODn//rPRdifzz33rC07cYnVVNFYjyKEY+Z6gCB7oi27VruQqfSQ9drU5kSlie+7frw//JK/LRSsurrGwZVCwVasuUUiAgA1oH93blsnwqWbZg+c5NNTuTWTqbCqykSxKmZscHTSrrt5i40VfIePFt0X47OrMlmbP7fT1lxxvvD3J/7pafvO935gnS0tduut14t4ETlt+HK5nOq8TjUBGqdYFLCkJOHjv5JJTaFxIHv6fHoBFAzGwMQU1AmrD1DMad0T41N24WUrFOzyzBoaau2mDSstW5Hg4qLZm2/ut1u27rKKcsx/xpYsmGvLr7rEMpmC1iWYxbMnRUe6GJM9ZMmTJaahItyhNuxPn3+8+N3vvmCnnbo0MTxc4iNStWC3KlKW6pQL7Qgpc/6+m0janBOYQt+7QI00CpTXw58bEUyK6obZVWtvsf6BARVramvydt8dN2vufHkGnRifkEzs4PPnvDrn4zNnePQrV9xcaoxQWiWt16w1NtZZ59x2u+DCz+l7Tz3zHXvyqW/a/JZ6u+ULG8UbCHMoM5w2gqJvYbyJmyC1rcSizbqbixgioiosgtqjmQ+LsGAqAPlrneipDt00akVoopXZ2ede5oTMigprqK22LRuvs0yFxyZsqPvvfcx+8eJLum9g3faOZlu9ZoW08pIivehlIe8+E8DGjJ/AFhJHIG3agLgzG1aeXWxrb5NClSSzcg5IBMghdAzfLUDGNdD53ynGng55O5J3YuLPKQQoDYLsQJ1elkOgsDdNTE/blas3W08veDX4ed7u2L5edfuKLPECVsSDLKjOcdpwG8C/nmZlbPW1G0Wj1olSX7gLLpRnM7bkhAX2+c//g0zwd773Y3v4sSdtYWujrb95re41uGhebk3zWCPVic2VzL3nhCYNHv6OSS8FkOL50biAOINvmBIXY1ZziJtc6U1bMVNuZ597qTpmWNimurxt3XKDwciLrGjjTVtt3yFK3rRHl6mCt/a6lYp5mPghYCqGKSWmUaSVgqFnz6FN4JIsgdZryjIP3bamKJECpj4nJQf0UllwuO1cMN9n8UhznNPuu4jXxIWGuY/GhdmuwLMGtxLezZq1q1Zvse6efvW7N9fX2q6dN8qiUL/WZ03RxeradVLByniaKECoSGlx1G6+eZf14S6IVBWJ5xQYMQh44aK59pnPfkp0rkNHj9rv//CGnXbyMlu0uFN0anrl8MVsJty2UjivcWrhnPvuZVUWLJfzThgBPtqYbr4DyOHa3D07WBVBb4xOdTTZlbimy8rt3PMut1GqotmsNdbl7datN6q8LZ6AmV276iYbHByWBauryduczla78qpLne8fbVJp4UMggusrtYZhOXhuCUAS6kmwGdnFU49uKfJwpJScfGz4AoEwqTpFJEmRI3xiFEViZ4m6m7a6pLaS6A+vj4fA+7LBeGRXrtxkXT39+vu8jlbbtPFa3xjlDiCRiaoZMgkjwWzJV6NQ6WkJVmPj5tutq+t4+r0Ka2ioFyO1sanOOjpa7JOfOlNmloCLY4I1IXLOZXMCmlLeWLIirpU341pYBLF1vX6XXh8m3Is30eEzG0SLDRB6dv4MQ8QYQnTWLrz4KhtJHT51+UrbsWOTwKuQTrl6xY02xgiVsqzV19baR/7nn9uHPvxBT1Ol7emB9ezgkc/l50o92ZRcO+4mYfmy1jFo6smHNxWJ3Gvzdd6tAsslpSu6UwV6iOL693kQ0XzAQkTBgw8jOnfzk1QhJj3FC2mxMEGUVq9dt8WOdPWqy2XJwg5bv+Yq158LkaCCYwFkCyx+c2tLqWMmINC77njE9uzZ50ui4MXZMvnqnL3thIX2d5/8XzpR6MjA2OEhEUVzeh2EcuuFC/NbTQydNILUv+dMW9+MiC0kD6vx5kkpOymGJ6hA7ztTxp0hiWCqBABZwS6/Yr1TyOAVVOZs584bS5ItLOoFF6+wTJlr9rQ21tt1668pSbUQJM1G61iTCLi5ZpWpIYKAaqaRrtRdWAusreKsrzy0qYhpAjiRZKeK9y4XonRMunBJICDVvLEQ6lWnUpceXpjxvr4+q63NJ/66CRCKFEUdKdPTlq+qtKvXbLajiCRZxk5/x1LbeMNqO9blFGJF3DKvvjC4ABSZS+yeJIT81a88a7/4+a89709SnpA9GmvzMvX/++99DjubmSAM8851VlfVyE3lESdOSKMTKWPIQFK5VueJ067ollUDBUp1Sh+9UMXChPXDlJcoVknXPho6FOJp6GLGJqen7LLL19nwiAsmsJluv32jmEK8fnh4zK5ZeaO6Xri+jpZmW37VBdbYWJ+yJdq93QLp2SSOXUi6qlsoiUXF4k9Oem2hIFZQ0TLPPLHTYf3EEC09iFS/hdzoJ9bLmhL2Gxv3CY4CRvyUicqcfocLUJBFPp6CDPHjk3+hpLnu5tusq3vArDhuH/nIB+3sf/h76bROTjnOz0KJbDmbNJneV71ykwX70Q//zb713A9SC5F5kakwaTVVNbZkcYedfe5ZJb8dUzV0ipl7kNqQfAqVjLPex/vrPHMQbSyJL+kBaayIl6rDWkARE7CUBhGT+noeP0Nr1sZELpyYARZxttwuv+I6G8CHp8aQ23deL3CKNHLfgWO2+dbbdVX8bltrk61bd40GNrAxSB1j7h4Qt0u4eWVR1PJZqXb4eFwkhJviNHqAE5b55y/vKEpdKqlO8QbSR2WokJoVsq7QkM+rqUDyImmjBEZNYKWO0tR2hAsI9E3pA/1psQkSiLFq3a12+FiflZcV7NzzPmMf/NM/MXYlpd1SO1OKntX/HsP1Un9aVWXefvbvv7SvPPmML1sCLthnNZV5W7yo3c694LM2gFxYdbV67Fx0AMq2F410f0HhKqlJO3PWeXze9qTYJQ0+ZuEduHLLhDXxTCe1Zycp2IgVPNjDiqYp2slDL79yvQJTMY4yGXv04S/YxCgzP8yefe5f7BvPfV/3xeZfvGiBnXvO3wvoYWGVVeF6RVObae2KjVLadLq+mfmBauWachmXzDNP7tJ9STSf+6P5AHpUak3izSXMM6szQ3LiibvNRXDS/cykScVRjEmSXlgETqmiYtKJyQnbcMtdduhIt0zW+uuusCXz5uk9AJMUF9Q4kBTyJ3yPVqXmlhaJKtRW5+3F37xsDz/6pCYS4YmVhmbM8tWVtnjRXDv/ws9pEfF3LDqxjNIwtRNFFO4+XlIkImqSK3ljI6cJV0Yc4q1UTufyeAewKXHVWeyyjDZXTY2TUBzV45ky9mw2G9aVsq66+gY7drxHz5Hq0UP3bnFpNdi1W3bZwf2HBSXn8zn7m49+2P7sgx/QhA8xmypcFSwieFqp9T4zd1WCk9lwMUJFC53EETL//JVdRS+0ZA3/jE9nN4cEiSDNFO0TaHHyWTy1IScqNLtesqOSFnXmZwnqTREP5ghUTOlexuy6m3bZocNdetB33r7ZMgValLPSveXhYvKxHIj3ElOw87kWsgvy6FxFue3dd8juuONhMVcjd6anLJ+vtPlz2+wfP/spvScPRi3XqeUZEMjTTp9Dq02dsIMo7tCdwzw4ZStpfrteA0aRhvTOLnzAk/PBQNTlgZvDgzoJNMxvIgnZqlUbNe81AuqH7tta6nK94sr1nl4WM1ZTW2nXrb7GqvMMJUjCy5p26WNbWUzkY4LVzLrwjAKMinm6cnFYsDQFK/PNf7pLZd3x0RHh7J0dc7SoAcWyMCxqgPwK4ngoY+jI5RxXTjVn2C+8nofKe0SKp0i7psb6epHppJW5zDZsucv27ieYm7Z7d22x0VHXguVzaY863tWtMnFbe6tj0gUX7yNvlpVJzYq3bnvEo/FS9cuspjpnC+Z22OfPPat0+jhJdOnILKv44+6BgI2TpDRITSGkfIg4OOvWT6+3OuHyAgQhaJVaRsbUYRvQKe8fVObIhlIQUar9Y1k23LTd9h44oh9hrR6+f5sXfjIZu+SS1Z6wZZBmr7atW9bLGmDXBBOnnr3gAgwMuhvz4pLrB0iBi6JNqilEql1iCX376/cWCWIYBshDr6eBsqxMZkunOBEWuUBSIXwtUOv8BfPVBaN8PeXamobADhwaKvlOHrgmH/NwKirE3CG6WnfzLtu3H8Jh0e697RYbGOwRT46NEf1uLmrkSo35KsfxNWAHiLSsTDoyW7c/Unp4oZbFaxfOa7eLLz1P2EOASogQuniiq2ViNuvqanXvwdlHWw8zEOLE9Oi3d3R446OkQV0xm9erkjcrBhD1WzJrnh56U8esQFFyJCCgGbvzrkft57/6rbue4rRx4r3nLmMXXrhSXAGRMatz9oVbb/BYIJl0hiV7FuLWhdgLy8VnKT7JmA3098t60mAZBaUA0aTg8fSXdxRJCWCv8tBZIE5+Hb3n2awWW8EWQgac9sqcbhqzjWaqWogSpTp2VcmspGmVIUYUYANuZMuO++2NvfsE2Ny49nKrqnJFDCL+uXPnWm9vt/h9mHuiUTBqmgoamMhUkbPjfT3Syt207eFSJOtgDx0nRevsbLeLL/mcyq0jzMqh0saJ1agSBBRzSblaOtNKrSR/htCR3FZE9TktOm3bbAoWU0JNqUGzVPhI9GtMKbUGzC/uM0rWOqmSP4XoMWZfeuIb9qOf/ruXbqen7aEHtrklmyjapcvXlizVkiVzbMVVl800iRDHJFfiwxbR05mWRWVD8qxiQ7ju3ozsCwuuRhA+876dq4twzcnvhoaGdcNNzc06ZWwAgistSNJiV2SMhPew5/IaQq+pkS4jovp1ivypPGGuBQer6lXU6afosGn73bb3wCGhads2rrL6hjrr7e21fGVOFqOmNq9AL4KRfB5LwAiQvC8SsmeZrF2/8Z6S7lygisQQcNXPOedT/6mowoNtaW627u4ebQQWX0UgJMxSB02oWChQUq48Q1dSeprN6p7AFbAexD3yqakti4VXL37aOPLvCXbmT8Ajspenn/kXe/bbz/v7F6bt/vu2CBc43jVoN2zc7nX5TMbOOutMe/97353qFR6QBtaRiEkJeaSJM5uGFVBPcJcY/IzI+wPFyzz12Db9fn9vr8y6JjAg3znOhMcaO9bVJRlSpQCa4JzznF18cadWCRiQP0Hsl8DLBXOl9ZYqfT7IB7/j+ey22x+w/QeOyjzt2LTWxidHxbEnIg+aFO+Zr8qnaNwnV/GAWbDJKd/dW3Y85sIJjhK577aiLVzQaeedd1YJU/fqmJ8WeAEekfsQhND04b5C3YprwISWxpmkBRQ5RYOKvFAliXBhDQm/T/AoboUrIThlc7Q2Nycl7kptjH/53r/Z40885fWfqWm7686bREP/2X/81h770lNpgTN2w/oV1tpSn4gkXq8I0Cj8tQLKcDnJCmhRU2XQM4yUgUiZI2OZB3etLerBpeCovb1dN0KgI5Rpako36qXHENrznBRhQt6UBSDCZcE1hVGRI6ifpxj45SjiuBLkuH35q8/Y7lf32vve/z778J+9x6oqMtZY16AuU8zf8PCAhuqRaYj1guhPmhwtl0JaODFht+583KN1wff+8Cn0zJvbYuee849Q9EvmNkgkWB+v4nl/XnXeCzDE6ywms2DYqPj56LSJdEnVskSAkB+PPJ6MRhp7KHcXrLbOhxPFEEDh/lOTcplcx+4/7LG77nncpssgik7bPbdvsInRcXvya9+2X/92t1c1c1m7bftNNlmYSDAwFctE7kzgTqCGKhKBpSRsIhBV35z+O5HWsUkyD912XRHzLT+O8lQFPnFE9XNyeRoAJEeKxnxlpcuGxulJ/eE8DFA9ImF0aWQFCtOucjHpUqUsDnGBFC6nRq2vf8TaOxdY30CftTfVCFQhnqDsSO86Pp8ty4WrgVEzU53gqdoCM2anp+yW7V/0DpkUvbLwbLh5c1vtwgvOFo8vGLNcC58fU5s0OEnux+VRsVDcBxMmws9z35SbOT16JggQp4kVGvaX5MSoafDePAusppetedppmEHiDDJlA637w0d6bOftD9oU7RKT03b7jvVS6F69dpONT7lJrygv2vatN6R+f2/R5n0JgiNeioYJXi8cgdgs2Eiix3n9QdZ4zGf/lhY+UjcJC6RZK/yd00+jfnDleEgENvh+HiILSbDFG9bV15dwb3xgCPFhmicm0wAclXLZOFM2MubBGgFJU3OTTU2OiWpMoSYw+YgHuCmkTzipOvkEZpzOyQnbftvjdrynr+QTxQ0sy9rCBR12ySXnCgZmU3M/nFriEs19b2jQQ+F/dbjU1np9IbFWgEVZaH4Gd48NpbI0zBxqGmk2nvDxVP8Omhgug0AQcYM4iQR86v2bnNR99A0M2+atd4uUQaq665bVet+r19wiS8RXS0utrVtzpahXDh+7mw12b4A4ZCkREwQaCVfC3WKlN7Jq5NqsqdrPffUOVec4NQFfhnnG1LHzAUwI+PhApSipVs3rWfyYDs2Hs+gsGD8bGurTQ6mqIlAb14Ai3gPW7vAI05XGRSnm9zEenDhOPBRlqURD5EReTGM33GSz8SR4hFTY+Jjd++DX7fCRLl+wZOoJ+uZ2ttglF39eboVNiG4OqRnRb2AToYQp7kDykTz8GDEWuTndujR8Ks+vdNWNqJtjXsPPqwyaKnnyqXQRkTqlmrhKpQwsmJy0o929tnX7/TYOUlqctju2rpE41OobvpCGIJudddbH7U//5FTxECOg00ZKuLzirtR6Hd8PX88aB4jm2ZZDz7FBMvfvWF3kwXsfe4UEh/bu3VuqrXNC+CgX7Eecr0IkR+XmExMym1oYhuPy2oxDl/y7KhUrOHWcMjVCVFRYXUOj97mn2vHSk06yPa+9qt1Zm3dql5vgKQESwqaTADEwRvTb4wLuuvdLtnf/4cBIPPjJZmxOe6tdcP5nk0q1qzlSl48TyGIp2k4Vx4CTQ1YV7r6gaYIEPThXsI7R4qBqLL4zV71FWhi+mLVeB/DeA7cibOYgdvT199r4ZNHWb75H/Yll0wXbvmmVmiCu23CHW5NCwbZsWmkNDXnXmJ+loKl4JPl6ucLUnuYTrD2IizQzYgBxJmdRvDNPPri5qFku5eVKdfBv+HR8ReSyfIh058fGramxUZOeQwUa0p/06Kp9Hhw3J6nS2tpSJwkVM77UKl1drWIOvppNIOVo2rAy5s2WVJGkLJkGBwFiJFCH08r4Ut/97p+/+8L/az/6yb8nUoSbMtK5OR2ttnrVlUltclJsov6BvpIrkwImLqC83A4dPmxnnNp7wtEAACAASURBVHGG7d+/P20cFzyk946v0RGkWP1gEHuoOFNI/HQtEtVIL/mCZsIeHh52EAslbmfwuGz5wADACmXhCVt5/Q4bROuvttZWX3WehgJuuOU+cRd57Y5ta62y0q2Gl3T91AaHD0EJAl9POJ14QeMr68kaIBUzu1gWLl2bgRMvOHNyUmkbAR1ADr6NXYOf53TqgZaViTwQ/5bWfEKmODm8BwEOE3m8uodvn3bwowbhYpSsahXxk+ZJ7EjtVhU2PTGu08PvifWik+vTJAI0UmtSBbDujMn68b/92p57/kczJAaB4UXraGu2Sy75vD7PpUhclQq0TeBTZaUNj7hvx2+KXZvJqO88AlG+R8Ap8inFGXwmQ4/QpZ10N8hmlYpXb59iFhhZfhp9ALCSTJlnL37JGihtnLDBgSERSYDAW1oarLd/xB59/DkFfOUZAr4NUr8oSxp7bDanpSW9H03PxAV54ciD7jRRUi7HSTQ6uMz7FZTr5eLMfdtXleRRiBbZaSw8lTAwc0w/1TAV+4FjBweFZXMDkiVFA25iwos2lZVqbyIXl79XLd/noHkg4mpSfuK9i4SNxe4c6utRkIf16Dp2TA+VGKMhjSP3ua/MdEWe2xEoLPBrew7ZV772zRmdPh500ayjvcWuXH6BTtro6LATRhIW7s0gBUXz3G/QpOMABOIWFoyUTGmZ6tmetlIdYFOxpG45/MTTg8c3WVjPnRl4QDXPMx9VNUPjvrzcjh3rsjGJPUyoU+bbz/+HvfTSK/aRD73f3v3OU0QjYw1k/pNiFfcUMKxKsEm2XDSwtLDMo5UGf5KlgTIewZ024z3brlV1TunMLMIgb6CHklgoBDTHjh3TYvE/pp5Ai0XjxLCz0GZXBC1JFMAPj045FZ6XVgl1Q+mivqFBwAbvAZefzhOsA12vnqZHH56f+Gw5phKs3LONnj4Yuhl75fU99qXHv1k6WREftLe32PLLztECtLd1iIeeS+NJXRfeewTpVcM/e7nWI2fSWSwULof75+HREsU4NJ4JQR6bxxnIfqLk+niPSUaCIVPuvQUQKLkmCUgkBlBg5vw+vQVo93FwYNmyOZmRg0VkA7uCd073jJXSGqVpWQHKDDN5S82sHrkHTyAkVbFkfb390jQQykpQeN8XVhYx35yuzrlzZWZZdD6YD+MEYqoxf0TGXCw3HmYrAhHMF5EvEiOcJAKjU0492d58881SH93AgOf1gXpFqzVtUJXykc6yZUEEqkwVrLW1xWe0ChFz009f/sDQoBb7SHePPfjAP5U2bUT3bW3NdulFn1WRgnQHISbwcyhU1Arw+ceOHUkyKv4wdBKS+dRg4YTK8Z6cZMQQCSxZUdI9CjwgvnJxQ0OOeoIjqObgVCf+HXT1oHFFNsFocg5DSTE8658xMjik9+BZzu3stOPHfXgTh0ULCzO5qVkHyOH0mVZtguFjR49plDmvDT4DUARunH/LJRDccWGcxDid8m1J/owXeTQ641cJHjgZHrABsLgfA3L1TkbHwStSmRUxA7B9Bg9wOggOxfhJKhli8PYOyL3gJubPX2D79r2pDbZg/nxh+MyKdxi5rtRdg9sYGR23W7c9YNAdImJnYdpbWuyiiz5tSKgA7iDAFOihIngsVlVOkKoIGIksIi4BSGZCwaSsmUrN+M8RMpqEjjk66vKnWBB6+FlUucBJ9HtqJYIk0Qj6DhNFjSd0YP8+65jToc0caJuzoMo0WkxoZOpNJMbk2rE+nOLWlhbda1hp0kDoYiIfS7K0zMYmvVTMQivwm0hzcxltysF94el7JXdGHo854oHwIVwEJx3zQIAjCDeZsxICVlvrKRraqtTgB4c89ROdyCxXRdsvc9Rm0g8eIgUZ3pub6JzbaYcPHxblGdmSpoZ6uQAsgEaI5SpcqjQ1OdCGFZuQGxoZG7ONm+8RgdHXwQmN7a2ttuLq88TH91nvHpNgTQBWlixZbAf27XV+HTBKmoAVhSQ2PPfOtej+E2DlwxfGSj0Hk+PumvDjoHYcCLlITYigquh+nWMp/AN6mmhkMSTIRBQR2AKqpgDQZ9UyVNC5fd74qSJPYvByaDra2/UssjR8pp5G75fM2uDIoAJ0GEu8J8yg8P8K7p56dGuR3Xrw4EEFVbX5Gk89in7jbAahXgzOZUGSXjy5Ovw4bi4qeMh0RXTP08BN6LSOky56kMNO5f3EdFFXicmcHT18RClQfW2dNOr5u/rFxz0VjNSPhyrAKIk0DY2O2LYvPCwlTPl350xaW3OjXXLp5xL0C7fcIV83s2U66SCF1dV5BYq4MaJ8KWwB4mBdamt9DnwaJYaPnanJ039OwJeIIeOjOvW8P/eIi+G1ZAFh2hXYJa4cr+FeuGZ+TvosskearsWfHEYWaWCwX+VpuI3CM1IbN88QYE15PYcSVDFN04TQGV1OakIt82oi5FAJPN+86vNFOmcOHTzo82KYA0NAQ15NLp9oVujEUzBhARSoaMqykxV5oF7R86Apeu/YYa5ekZFPOnrsiCJUvtfb22Mtra1aALIJ/BI3m2d6hUZhT1hn51zrp6M2je12IMSHApHH8/6UZ9ffsMuZp5hCFSMKWvgVKy5W0aeqslqdfDKfAmO85RndOFJMABBNhEIFKxVgSgBIykBYRH4XtxTxgIK0NJYb2RPuq4Q5CIhCQNEbNORXVW+fKEHEXIkvSnD1/f5kuczJFHKnBReVAtlUgJjyMKXS4hk6stfY3KTAT2BRUvEkm2FThJoZ8ZU4AET1BDKB3ukkFoulQobSq64ulWgx2dJwTaO6XfKjwnJV1TJN1My5cTYIX5HqiVLMOPGmJlmI+JnAG7FyauzwYachQcLg88gI2CREvexyfhfaFXPaBSyl5kJYpFu/8ID0dOS7U8Nlc1O9rVp5hbRfVTYuEJn7MILpwqQCJzIJAKnxca9gaQa96vAuPe4pqVfyWHhlJpWVCb93AcV8jc/VQ+SRe4Eyxu91dnbIiioDSkicov3ETYiN5fyGGfkYZQjQvVKgyXNVYSilnd6945E7VoKNxJcXrmpLimOIWJGFsFayPFUuRhl9jZk7brlKvXOc4qVLl9qBAwf0oMLH4X+5ccyc+wrGfo4IPaJCJohUzQZAlFnNQeUC2MWcgCA6AA719/dpNxK88OVRuqNOXKBvnhrr7JxjXV3H3IRly23JkiXCErhZFonNyBefic/dvOUeG5GQkpyH3qupqd7Wrr7SpqbG1aXLPSxatFjz7tiIPgfOu02HBgls/RipxQsRzHRCuTpew73weQ445YTq4fqQceX7lRWeQxPn8Bp8O6cZ9IyDwCbms0WuTPPwuKbgJuo5UuwhSE7TtLQOafCwIOxU4FETaUqT+VMVRBXDnOrFe9U3Nsq18vmaZJ3z554HUcUdPbBzjRQxyLV5QVSywgfVCfmCkzeskRqqX1d72bWxqVFMj4qqKkGRLc0tQvZiDCe4tZdEvcGClIyM4KSlJ9rhQ4dV8QIQUt2aGfSCdGlxctIlG6Cnpzfx5MgGhtEjVhwRp3B0ZMx23v6Q9Q8RiYsCJ1OPysT2bTeL0/fWWwRxXtIFTSTadnSNBgrH1MmDfeNxj6N6+N6gUVBXb6RGkQcPDwwoiub1vA4iJCDT5Dg8QUfHQjc/3AfPhoWJqppQP4KytBmi2zbiBJ4dC8e/OZgKvtM4E0G4QuSmZCUJ5KIoo98vK7P58+cp8GSj5MBfqiqtd2DA0+aHdq1V349gypERW7xkiXYoH8omqKmu1oPioXd0tCvoIjjgZKjzVcN33Q8TQfN9plRwwVTj8OXKy1nQqry+DyCxZ88emWzmx0RDJic5YFz3847wMYMWc8rNNja3lJo3dfNl5bZ9xwN2uKvXyQoSMTQt/FXLL1B2wIZgOLBSoFT544EQvPo0rH4bGhoUYKLMJevSIdFBrJsjJUq8BKGOlRVyFzx8Veum3NVMjsFBdHcZiCDP8Y9TSd7P9fm8cYUTC/dBAdnUlDaUroHa+6zysdLrRF5l4/D5mH5QVoLzUO5g4XHPXJMscHlWaOgodDYi/3u3XVsEg8YUs2vmz5tnBw4c9FNAwMaAPem1wsVjisSw+1EK/0PEBjXin/NQTznlND0g1J727d9X0ogFHQPpqqqu0ebp6u4qQbPQmzw4rJArwG9pU6UCDuYKCyAs3YpWla8tVZ686FBhd979mO0/1OWroxJrRgu//PLzFXfwu+IMjk/IauH7sFyaDZOrUPZARTIfRJM02I+NxP+AM2wIOAccCj3MfLVP1NB0aDKAvHrfNB9+2qN1FW1SSsufvJ50j4yIwJb3xcosXLhQCKiyIyZWzJ0rF8DPgvdIhM+z4ftYBtaM9+HeOHykbaScvBfumc+m7q9CESqflWzwPuvonOPj2+/ccrWoV1wYaBbzVkgdADHYfZwI9a2rQW/Cautq7Pjxbgcp1EAxba3tbfqgBQsWKdh4Y88eFTuOHDooszw27sI7oF7sUuriUaliUZubW3SiOflAsTwAuO64noiS+Tz52dS3xg25WZ60+x940vbsO5gWHuyaIQaNdv26a7QoAEbsekAkHzgMT5CT4DFKvrbaDhw8YFUpwuZ7nDYHZWDo+hcnU6kX7WRj4x58DvQpI8iD4jHQgGKMmlK8hZnTzmcr4E0NmNQ6cA9YPT6H585z4b6BxTnFfAbIHlYp6FZ8NoeR9YELGVQyFj6wF/7OBuN5UW3kT/7NpuU91QcJzsLCk7bh8BU9TkyKY0dAwwvZUUqAKP8Jqhy1uroal+lqblVRprwypwAMTdr9Bw4odyf9Q/bTOZBOoYrgiL9zs9w0sDCvJwBbtHCRHTh8SNaAYKmXacpJDIFNwyaorW9Q1B9AEzoCTz/zPfvliy95mqfGTZMcyoqrL07TrEflQg4c2K8HXFvr0Ce+kWvp7nUixwAQKrl6UgHhZHGSCHjD9NfXU2MYkHii/Pi0y6SjOQdbloVXrp1m6bCQPF/undezCByCUPrgOfzud7+zBQsW6FnPnz9fr6V3QSc1MaJwURS9+OJ1In3W0z3r2YQDaTmBTcIGxh0yZkNw0gX+5HL23ve+1379619bZsu6C4oEZUCP+CwWFFRNAgIELUmNkg/yC3YVB6/aHbXGhkZbcuIJYsP88ze+obo2P+fimhubBLm+/oeXtePnzJ3ndeK2NkXtdXWgdAM68ShO8XB5aCwOzX0e3abOWRWHYOb4BGeEijiNVblK+9mvfmfPfOP7LiuuWINWq1q74pJzlCU49s/UKm8I5YuNRHDpKaW3j+VpkEilUzYAnT/4YQ1CTNOriYNA2PgdlULTtKmY8Z4rc4YyMDCmVmlwKnhFFB9FG5nuoSGdcmIfPjMCOw4SGEfEFqxFYChYTDYk+sNSJEupM5uGU87mYkPx5VIxno3xfKlUCrm7beMVRXWKpKiWF7vSlHetjAwNe5cpxY3UKDk6NqICBf6VEmVXT7ebqrq6ks/B17zx2uu2aNEi6zp8QAtOVK+IHV6czJM3aipTqHH/xRc7GdE/brC+vtF3bOpmxdqoKpZQLJC+3a+/Zffc94SnYEp1WPgaO//zn9am6uvrtWUnL7O+fvrwHH3ErXCyiFmGR3zYMf0vge4pVshmlbLxoFg0ngMPlX+THeCKGuvqU97tDJ3pCWrt1Md94pboWKl3TmlYCqSxKirjJiYQ78l990GBIzDDNaFUUkWxaqbeLiJnoWDHu7ttlIENCbPn+fNe2igJ/Yu/x/eV7ma8Uph59I71iuoxXYJqCVwgJPb3loR5hwaH/lPbNDm8LECuPOXUTvUhuuehMsWZhwKGT7GGUFC4dch0UCiYnrZFixcrTeRm65qa/T114jw7EFN3xDdepEDUrQnIGpo8P+W9D3X12l13f9EFHBLwAfNlw4YV1tfnwBInWxTwXKVONy6GB0KARCmY6BkiZXtHux3Yu89bk2ZF3XFqA6lkk6qZos6DUfRllXINDft9oGeT3Bvv5QIJ7vOVMZGTj4zIDQR0G3FMUNtb2to9xUaGvabG2tpaUg9jTgeJg8nPAbckHZtIGuSZpGz+5RtKI1nT9agY9MW7bxQDh2I+vp03Y4FIT6Sn1tMrvx4dMyw6YAonulDEV8OQpeFwyoZh7wD0JNVHTKxGh4F5T3jk76bc+fhcKEFOV1e3zV20yF5/7TVra2lNPpLFB+BgFq0PG3D2al4na2IqjdwqFm1wrGDbdz7glOM0mQGLtOLai8TKxczjUvbt22fz5813AEO9Zk5oyDGWVFQpD8gIpvCVjkm4v44giWcDs1gyY2lapSt8AvBM6V4HBgZF/Y7TzObGYp104ol28JCPMvMEpCjAiwBOzzxZADbHsmXL7ODhIzLdYPRsVKTZOfEgkDzXqCdESqjq33RBPzv99NPlPl555VWflVeeJlNZRplY5skHNhWZ3X5w337VdwFROPljI/gCKMyubQe9mWIGN8eFUd3iQo8cPqIFBIgJuhTpAj9jgUhH4KHNLlQM0ueeWLv4IoI790e0ZdUpz/Sghn5296XkufhbfBQ3XyEKlgrRNjA0bHfc+VjqX/dCECfkkkv/0UuUkC2ItDUPjyjegy2weqwHWDhVPRYo6GROpXZBBixE4ApE1ELIcj7eFGtB4DU+MaZshw3Ha7B6vI4xqd3Hj5fMNRaD58f7RyoWMK2eX3m5pmxj6mlYIZClfqLIvTwj9PGV3X9Q8ByQeBworFkmETKGhgeEFH70b/5ve+WVPyjOwRKQdqq6+aV7b1JExFA+ThW+Avwa0uNbb71V0nalGAIRAL8DnYoNwEVxkpwckU8ivFm9BynOosULhVcP9PVrE4AVYKIo1/Ilc79okS4KdM3fF1yd0qVTukh9hEgBJKX5N/hsGh85daSU5RU523TLXV7ISHAm17N8+ee1gQjIdJLLoHwPWVNrs9OnoECNg3Hn9XnBrxNil8yyePXFokypQ8KO1g0yb0aTKpzsSNArOLYwYVXM8ZNoErJsY4oTsKq4Ew1KTPIuXFdYPtfZcUAM9yRO/8iwm+k0hgW1UVf28InaYY3405FIpnJ6O/fChfM1WetY93H78Ic/JGyGQ0j8w3VnvnzfzZpJozr05KTKosLAJ6EF9WsRPQqusDmdXjsHBZLPVOHAmzD49wknnKBAqm+AzeCFUzYF74OvB3fHPNU3NmjHHj58SJuFgUR8fmDtRNzk69wQn8vCn3rqyVrY3/3mt7ppzLI49pr5WrCtux71lqfU5oiPX778ApueZpqFyarMaW93WlW6J6BZTljQjtU7l+bJKU1i/HdquCC1YvHJrUVSUarkEjBu9oFq6eLxfJ8TqxSO/rnBQVGnAaWcdeMkFlkVJlkeOpKmZHvAhyHTJkqoJZ/rC+uEjEA0eU3w6LznYcqytLEVCiLWiOGUMd1zjHANelbm649tK2LKtFBJBgSTD/qEmYcASSBDdMzDBDtXVwupwZDj95wW0gsRKnI523dgv33gAx+wg0otZtIJV7V2UQNep+ieIcOkbYqUY+eip+NdIJHiUUNXIwUnPJWBMeH1TU1Ka7bufMS5ZIlszLVecMFnLFdZptFkkkPNuKIXlTjvGBrzGnU265y3JIyAb4+/q+w5ewxZDERQT2G9FpJoHXEjVdVE+vBytNKzEa9A8miF5kFrS6eeXFs+e9QXvKWlKU3HTouMRKoCYub8EARSLPLSclTrWFzAL1Gp4RFMOL2d95Vu0ZQHkVFj8EOTdSIGIAzUIC5q6dIThfkeO9ZtrW2tCqzA6WUVYp5qIuydcMJJtm/vXsGMXr50rRwujJtvbW6Rn2GYMKeEoGg2jEjMgCUQSlbFn34CeWjE54HbRx09KmMsWrQIEfw1NzfZhk33KkZJDWtWna+0Ky+/yArTY3bayafZ7t27dQ3KsS2NRkuEC31+0ujFtQB98llt7e22f98+neQ4XeIMJhPPQgCB4sJefWW38nEYRF4hdE49G5WF4P34s7Ozs4QlsKHkgoRquuVUrj86at3dXcIgnBQCv69OmxP8JBRLmNHHsw7Xi/VlMxIL0a0r2HZkLE3ldqSRz+E6M4/fs0GmvhJcuhzpLm+KBIXjwR/rOip8ndmsPCA8F5RnLrK3p09+n5vid1h4/mRXcZMEJVJpSpuKG+Xhc+EgVSBp+HdV2sYci4cRo9NS7Qxebgy3EOlUwKaoSjj6VWZz5nTY6ut3ajChu+FpKUlcdvH5lqs0Wzhvod4Hl8P/pHf4dnw+zJuu7m49JK7t8KFDRrDLn+oM8qPq6Bh074YGReKwd3SKUtqUKy8T0tjS1KDnxGZQYWaqIFOvAk4isi5e7OVhfs5zBDDzlBCh5xG5ymgSZfGpYbiuDfGFN65geTvnzdV1URmlkMbJ5/V8Vv+gB4gEyzzv/v5eXZMX0fos8/hd16uLmh1K/k6q45Qd998hPBQSH1zsgUOH9YFwvoQNDw9qIXmo3CSRrgMLznFTE0SxqEieDwU7P+2005ReschRueJ3Gpsa9CAYMBiVpYghlPfWeQziIIr3qhFNf/FL37Lu3gGN5NCEiVzOVq+63MYV2HlxRtBdkl/DuolnNz5uy04+WYEsmwMkrSTHopGiruilzCXBrYoLkmvUYWDTV5QLJm2sdx4iETZgEQ9atXTIGslP63SDDPb36Rr4t/x91nsTCaSPH+9RysnP+CKdw18oOG1qVpoLMQX2sFrNAvXLlidhSA9EuTbdV1LRBK+ZN3++Zb5453qNJglcmoALKBUT3N8/oMUMhg5+ROVWsWkdcePGYZLyxckFatzz+htJF29cpr2hsUkLD6QIGkdEzOsw4SwqlTEu3OFFpx+B2Olk5fOCH3kdOW0ENjz8qPVjcVj4o909CmYwr6SUVy+/wIY0r86HJQDv8loRQFP/GVbjlFNOsV/+8pfaLIEQirac0sj4XnDxFBWnDhkwdbFsUutXZwdwdFdpkUOdCnUQUctQDUsR/rGuY7oHClq8jnEr/Ly7p8eWLVuqg6EYJCFydQlt1ABFla3x/04Jw1KiJ3Dg4EEVYYjRgqcYAR0HD26j+PWP3HZdkXIlUXx0XvDQBgcGBXzgD+YBeowSJdYpNaqpd9UMomi1W/X3yULIVShSLZeZyedrZaZggAqwSDNiRsZGZbpY6JNOOslee+01ZQQUQyicvP766+n389ooLHy4iKAzcVNBGmHzPfH179qbbx0QCdPVovK2/LKzrTA2ac0tDTrZCxYutD1vvKGS6FuJ78/G5CF55uINCxFb8D3BrhMTdvKyZfby7t0lBg3Xz7VF0AYjh40xt7ND18/p1eZJaKHLrngJl3QVi7d37z4vswJIqWbP73gAzPOL6hqDk72+79mAtHlF1/LFfdfpp9vLL79sdfUNSuUIltn9vCYsYxwULI827m03XV6UGTSmOfbLj0SPHHktfie6QgFYSLWYncb38IEnnniiHT54wJYuPUk3jAkiAkdJGk1WPmTu/Hm6gFdf+YNuCBkx0g0elDhwSVQAHxQRaNCTeFj8bgR4InqmICjydn722JPP2t69B0XChEgBVezq5edq4Wtq/DMwr4J5wctpDKUMevRoKSJHn0YpHOzXRMNS/AOBIaGSLBTXwCmlhkA0r5gEhJD4ZWjAq4h5ytfHpQg2o28LXa22VE2TC1Cw6ILIuFYWnqZLDpqKZJmM+A5Y2qVLl1lbW7v9fvfLugZa0kBbeR8KbFgv6OgLFsy3ffv26nPASThYUeDRCFa1UG25poheLaeeKD4wXo0T08NCCWtMgYMP55vWCBE1WKZmymmEjxgSkPdZsyBi4qGlliWoSywE9fz6hnpZADB3AidGjfUPDBr1gNjpgfJhbQQBq03awRlAkGh0ZDHxo2WZCvvmd79vv3zxZXHKYdYCb1512XmWLfrkCLmmRElSPSHx491v+8PgRPGemHwCOSzNbJ8vcIh2KLV5eZ4PM1fl5rExzXg7uH+fglI2GP/GXLNp2GQqG6fBSNGHCLuI9q7ow2NDAYodOHjImpuaSvGGqF+ogNBJm2TbyPe5D96bTIwdxqYjHti/392nGFKDrunPa5llK32ie29dUSSvFfm+ucWOHT0s8QB2fwj1xWkTzxwevSpzMzIbUIx54+a2ZlGCqem3i5yRZqAxpntoUGkh/vTAoYMGpRvMnx3Z1wfu7L43SrpRP2YjCeYcn3SZlcRa5XNYiGE06spy9h8vvmTf/+G/C/yAZ1dbU2Vnf+aTlq9w5kyAUUDLasdGIjU1kODmRPzUTLnUHpZ8uNQvEnE0zCaY++EjR5KlchYwGQInv6ba4wi+x/1Qv4+NvGjRQuH/PEOuHatIDYMNzgKxgaLMirVgERU/JJYubOawklw7B4vf4X6Ih/hZBIsE0Pwu38NKidUEIol0HPf44PbVAnCii4P55OTumOkaATW0D3t0yf+cAhC81994w1E3RBCmXU6EDhnBqML3qyxfjVBCmTU1NSp9ES2bnH98rCRH4qVCJk95vRlfxHuRu3reXukl09QCxabDrImGVVll+/fvE3y7+4299vgTT0u8IauFr7ZLzv+MlaXxKVTBcC/CABI/X5Tkujo7dOigTjlwJ1aOzIbXhK4di0MPH0GbyItJ5NDr626psHJsRip8AEsLFiy03/zmRS3k29/+dqV6eu8JRBXrFZSxIKR2xC08B6hgArTGx/VZvAfvSdPo2962xPa8tTfFOs5o4pl4EDolCBpLRPEMXOOll36n5xcnPdwGyqWsRWbbugvVUEEKhQlBQlMPRHnhuI1PTAlp4jXC4EGOxD33Sc+8uQr7CdQJoqAujLZdSYVOKpI8cuSwAsXDR48IyGCnc4qJKagtc8qxKjRa8jvisA8Oq+yI9RBF+m1L7K29e62hrk6Vw9bmNqVik9Nltv1OKnSwSgtWV1NtV1z0Wf6hoBKzPFtiFPOIxUEMghNI8Id5F0rZ1CQSBEN8hQam6pznw4OJPu5ZTrOwWAAABvFJREFUTGDvIHROBfCYJEqgRNtsXII6CkFtczpkesEh+JMvTj6nSzP3VCHEZ494Kq1NjwrYkAYl8jwbG73rlWfMurBxJLyUAB1laalbCYvgKGWSgU+/l9l+/cVFpLkwt21trfIvqnc3NGiXAtzQphMa7ZxoatZAlbBOojLEQ+ADeRBcAOkaqYMHRpzgCQWCwqKtKL5Z+G8CSJBCHoT8N0SDnm6dlob6Rj3gI4eRP81aY1uL3r/ryFH9WZUDSCmz8SmzGzdvV9Mg9KeafM4uu+AzVsyWWbWUpt2PB4YOTCuzy8ad1TDJ94Jq3tFBQ4e7lEhf6d1z7MERShaH9yBd4/5h33JdsSFU+yZAG5sUlgDKScyDBaFphA2BWed5UzvH2vL5xFguFU9KPKxaw/HeHnvnO9+pcSxYXiy1KqkpLS5RvmYri6eFn03OEPSNjxdAAfOSC4S7pTbfKevp7VGKBuEShA5fGcIIAV2qNJoeaHdXl0622q5BqdTsT8BHKbU+FS/qrLe/z04++WQtPr/PotTVNSifR6eGWvKRw4fTA3YtWKLd4eFxa2pDdRN/6Pg7o8zkGianbMfOB2xkytUr3vOed9mH/sf7LFfmvWlsnkgh2XD8OzIIrAlLywOONDFSOR4498TrMZEshuoMtEez4JWV+v67z3iHDg3AixdVvPERq4e76pw7T344MqTFixfJXfG7x4/3yvJkyp2AEvgIm4nMig5dxz8G9WwCKY0iFu3nsjKTE3JP3O873vEOcfkWzsciHJAb4Xq4LjZV5s7NVxX5UHwPPogTTQ15/779DhXWNyilU5ExhgmlZgF2rwgEaUQJf8eEE8k6ScE7cpyPRp8d+Wmda8tHg37C9slJA1o8/YwzlGcTmLS3z9HD7ek5btlsTvPtcQ9DQyPCEQBlvI5g1j80Zt954Yc2p6PFFi5ot5amZsunFqpAwBSApdZh3pdNRZFHRNNUYAnXFVg69+DFEidYsrD4V96Lf3Pdbz91qcz1q6++6n15GhA8LkugBpMCJW+v2EEqpTNYm3loWEr7YskyRSs9D16HYASvI4/n8/k8ov5onuBzvf89uIbetctXXC8CDX64YA6TXeS9d45OGrUhJ1YoJowHQu7HLzQ1tSQz5PNWPJhw3pZy/ELBWaTqb3Mcm9ewu/g5fx8ZGnS2SL5G3ZpUjCIHp3BAIAN4I1p1olmJk1dWJloWppj3amlpSxOovd9eqhaa+Ybahte6OXHeIQOciYS3B5R8EcCSe3tFi8qYVx65F+IINgHXHac+ImbftB4xhzvq7JxnR48csSVvW2y/+MUvbPHCBXpf5upQZqbRI049+Ln4c5U5mzOnU00msHZEBqFRNV+tE8n6+Wn2AktM447NiushnuF68f1oBcxUL735MrKgzg5Suv26bz4jJGe4Rlk6miZZdGrF+DOUKKKYQD66YP5CmXmfHu2Nj/gYL0WaokgCQ1XUph0z5mHGqWEx0cKXJhEQYxrnIXp2InZwgbyO3yO9w6wRaFEDj5vmmubNW6A5LgRAMHz5OYvOaaUbd+68ufbS715S12N9nevToLXHfYHaqfxb6uwdV0ApBm0qnvCQhN+ndIx74Wfcc4g68vv4V1q3+KKoJe5bf58CrUWLF9jvX/q9vfvd77Gf//znej9cBfcWamCSXU2jzvH1WAbFRF1erGlqbhRtvafHadFhBaiJ4PP5fK6ntbU9PfdpweE8R3EUYCtPeqDKCef9sTqk6/xcXUNP3HdzkZSGU8cNR3QI4MIJoFIlKtE0rcXO62bXExEvmDvPiQzlTg6I4gUXyqnhRr1Jo09/Bh4gaDhNV+CU4tvhe+MigpoEygYqxfu4C6AChabulDZM6NFyoufPW2S7//BqqVWrrtaFF+hY5T0nJrwVKXJZpoY5ROqyZgI2YNGWO9jBZ6jXL6lhuTy74+xBjOT3+Z8TxLOb0+6Wq7mlMal4e4eu9/oPG2JEFLJACjHv3Bdw9euvv6YYQPFKuReX2Ozx/vxJ3ULo3OiwGik62zt0kHg9hTUsAxuUplfiJgFrYfKnJ62ttc06OjqV4jmHcdoyO2+6rAhIAbAC3iu0h2pRahkGWXPFZ4CC2pIejqDMcl8U/G5UzXhg7PJgfCiKT6adm1C78+SE0LtIMXpT+dWnS7nsGj8DSJJ4YqI6QzKMmXFhJicnaSHK+/yY9OCERasbZkhB5Eu//40eEE8rfDrXiRuJiN3h6Ua5HDD7mKnnCCSl0y69ln/zu17r9tHoqrZJ+AGk02vkyIuhvBF1dgQLuIbe4z0lxhKHQSVwMZCnbJA6SNKpjYIQh6e52Z/HokULlAIDu/K5R7uO6WBSyeTZxrWRfkd8BTfQp0zOVDsJ+v4/WJZZZ4vk0WIAAAAASUVORK5CYII=">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -610,7 +637,13 @@
     <xdr:ext cx="304800" cy="304800"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="17" name="AutoShape 9" descr="data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAO4AAACzCAYAAACO/iALAAAgAElEQVR4Xrx9B7hdZbH2u8ru/fRz0kkhjRBKaNKkKCjGC4JSBEVERLkowgURFDF0RQREpLeLqBBCk4RAekhIAukV0nN62b2t/j8z31rn7ES8/733+Z9/k8Np++y91re+mXnnnXdmSXNef8Lp7e5Fe9GE4QAOgIDfDwUOZEkGJCDoC6JarcI0TehWFY7j8MeUFgVnTWmE6VhQIYOebFkmbKsKwzDQ0NDAz7MsC/Tw/u6fvpZkSJLEz4Gj0v9g2zYcW4IMFTfe+Av4/VFEY1E0NdbhlJOOQ1fBxt7eEtq7OpHJZVCsaNDLVew90IlUfT1s00IoHIJuWDhQigDBekh+P2RVhRrwIxQOIxAI8HN8PgWKokDm07XhUxVIsiQ+w8GktjiuOi6C+qZ6xEbNgG6GseCD+Vi0aBG2t2eBUBKOraOqaTB1Gy8+di9kW8M11/0cPUUdtiNhZEzG9791DqyqiY1bt+Hj9Tthpy5AJpNGqi6BUqkMNaDDNC1IjgRHTmHbrl3QjT4E5ACi4QiGN4RRV59EPBFCa3Mr0uk0FFnB4pX7kSlbKJT3IKBYsPQOSHYJFcNAUFExcdp3MdDfiaOmTESxlMX0KWPhOEVEohYCko1oMoU33liBbNGHxi9+CTvrfbhg2hh8eKCI7v4sUqYExTIxkOuB0r8XqR1zsbXhHBx53NGYEMlj1iWnwDJN7Nu/B3975wN0ZDVojg+5ni7cdPU3UMz04Y677sT4YSMgWRZUWmjLgGQDsB1ICqCoKmRZAiwH9B/9oz1A14WvigLouoP2TAH5ShmmBfzp7p/g5OOnoVAoIBwK0VblPSY59Fwd5XIZjmTRbuKtJdF7ObTDh/ai7dA+Ez/zfk6f6eeSIiMcDvP7K5IC09Yw85qHUDT8fJ0cxwb9pzgWTEnBV49twN0/vxbxYZMB00CxWISq0N7y8fnRsRm6zucFiXaWeNDep9/9V49B+wAgyzKkt2Y/6WQyOWzp7Icl+wcNl1ZOoSdIEhTYkBUZlUqFl4CMk96IDDlabsdV5x4JRRGLrCgqLFODrmmQZBmpuno+SV4MOuBDFoh/DmnQcB1bGXqeA6z8cAU2bdiK5uZGdij19Sm+MJFkE/Z2Z7Bu01Y0NA3Hph17kC5U0DOQxojhI2HoVWiaDsu2sb8UhRRuhhwIwOdX4GeDDUP1+9h4fT4VqipDVRU4tskGK7MhO1AkCRObo/j+iTGkGlIIDTsaVc2PVatWYv7772NvXxGGGoVtGqgaOizdxnOPzEK6vwO/f/Ql7OrNYlgqjrOPGIZhbY3IZ4tI5/uxZ38Z2/om8xrGolFAlmCaVciSn51OxVSwcfsm6KXdCPr8GD/2KMiOAUmy+QOOBU3TeHNqcgTxpsNgWXnA1mDpWSRiQYwd1YrO9n3Il1vQ3t2JunAMra1taEj6AElzHYSDukQMjlXFTgf4bOJR8KlBfPmweuzsyaKnZKLvQDeGNw9HKGhDzqWRmXMPIufciExJw5cOT+LSGS1oSiaxp6MTj771MYJ2FkeGu1Ep5dE6Zhq6s2U8/sRTmDxmNMjiFIlOlyxTGJktkbMkw5XF9w6d39Cm5o2tSKjqNg4M5FA2DBiGg4WzH0V9IohSqYRQMDj4N2SIWqUCTdc/13A9I6H9WPtetYZLzkPx0f7ws+E65BYkBV/+3v0oa2T4Yi+zgbNhO/jzHRfijDPOBoJxGOUKBy+Z7Ef187nRg+zCJudSY7i1BsuOxwtiroNhh0bH4P6Ovpfefv1JJ58v4uOd7TDVAL+GLCu8ib03U9w/oMhpOxYdNUzLgmNr+NrkJIZFyogn42KtHREt6bmGaUJRfUgkkgd5udoFOtRwLZN9ED/f0DTMfvVVpJKNqEslEYtFodBx0YlJDjp7s9j2WSfijS3YsrMdhiWhUKqiohniojkO9GoVXVoEmq8eaigGf9CNsn4/G7DP73MdDtiAySh85IBUivw2VFnCqKSKH59aj1R9EuERx6JcVbFyxYf44IMF2NOf5WhuGQaqugbTsDHr5h9iTHMdHnr8FazcugvHjW9GW1TCKaedgo49e0ExoD9Xxd8WWFBVen8/VCXIjpIcBjmPiiFhX2cnejvXwjIKOGnGOZBs2gAWorEwTKMCmyKF4+CzzhyUSCtkjkwyRxafIotNSf98QN+BTWhJtMA2FYQiQQQDYcDRYBsSHLsMnz+AhrNPRldrAoVCGjNGDUMoGsauzl70lGRs+7QXMnQ0+YH4wt8j9MUfoGJJuPCYkbjy9DGQLBu7u7K4YUEPDi9uw1H6CoT9QG9vHn2ZAhas2o6Ro8bCJ8lQJQmGbcCxLMgOIKl05GDjJSPwHLzY3IT8FECVkC9q6C1VUKjo7NzWLnwRsDTouuH+rRtJbRvlUpn34OdFXEZ+9J/tHGS4nhF6hhSMhNiI6MOEhEy6iAtveAqGwZtUoEmpAtkOwIcy5j9/PUYefipk1YdiNjcYSQOBkIisAO/LweD1OSGWtnZt8KX3ONRw+ZjemvO0o5eKWLvzADKmD7Lih2QZcNjKIUI9LSihGItgnA4TCvyOhiObwzh5HCAbOi9sNJ6ETl7MMGFZNgxDh2QbUANRROMJOA4ZuwJIBrmHocgqy3ywtkUeTHhdOuAP3p2PSCSCRDKBcCQElY2JsQW/1qKFq2H7gkikUti4uw+VchWG7aBUqqJa1WHLEsqVKhw1ii6jHlI4igBB5HAIql+F3+eDSh8EiSWJoy5DZFlGKKjycRBSaw368NMzkkg2tiA+9hhUKj4sW74c8+fPx/6BAuxgHJZmo6iVYRs6rr7sApxwxOFYsHgNnn11EZriCqaODHO0PebICbBMA7v3d2PJOh0FNECFClMvwbIcyKqCgBJCsVpEpH4kdu1YhkppP5pSDYjF63DFhV9Gb18/PtvdiXK5gmAohO4BBUZwNPyqCsumjUZe20E0GkCpWOHXHejajrp4HVQEoUoyTNPgcwUIIZl8/kWninG3Xo3S/t2YOmk8DEXCZ305pNM6KrqCge5u+GIJNMx9APqkmdAiPtw+82hMa9QwqmUEdnXn8KNXNiNo5zHSOoDj5U0YGMhjIJfHkpWfYvSEKQio4Iir6yZff1Wha2ox5GenLLsGYVJEk1yoTNtFQrZcRW+2DMPUeS+u+eA52CahP7DToy/IGC3bQqVc4c8SuUk3Onohmd6XIPOhhusZI6dpcBBLJIZMyzbx4uyleOqN1bAc4VzYJmxyNgZGNIbxyu8vwvBJZwOOD6V8cdBYfX6K2oBj2xzMhgzXTQ9duHxoQKu1axGFh+C09I83nnEqpTJ2dfVhX7oMS/LxG9hsHAJPB/w+vrDk4WWJFkNGWyqMeuMA0rksdn66E0FJx29uvgQWG54wStMyYelVmI6Ozv1VTJwymhfRkil3FHBI5CQyDIMWmAxXZMtbt25BYSCD+vp6hCh/USWOtF6ebNkm/v73f6Bp+CjEonFs2NODTDqPctWA6g+gVNLhyDIqlOtUHKT9bZDDcTbcSCwK2afA7yeHJENRZAHTZN4f8PtUBH0y5/h0nC0RP244I4mG5mGIjjkKhhnCwoWL8N5789CZrcAKxmEbQKlcZHh03lkn47KZZ2PvgTRu+vXT6Ow4gNOPGQ6fz0HE7+CwEcOQTmexaUcPDuTGoqrpkNUgZN7EMmQfIQoTajCJYv9OdOzbgFhYR2NzE1qTEVxw/plYt+UA1n2yw82f4tjZVYaqhGHLIYEiZAWOJMPHMM2Hgd7dGBjYiqAPCPqTcBxy7WLj0LUNBANwNBNj/u1ctE6fhnFjD0PBtNGXTqO6rwOObaA9b0DzBeG89zSGn34xtvRm8eSPv4rprT7eFzs687j6r3uR8pvQynlM8OUxrOt9+FUFz85ejCOmTEDYrwjD1UwOQbQfac1p/RlJ0abgvUZG7RPBw6fCtG30pHNIlzQOCC1N9fjHK79DtaLB5/MJjOZyL/S3lNZxoIEFmwy4ZuMLwxWG5BmLB5+9/UVPD0Wjg7CVHOH1v3oaa3emYdrE8QjHQq9jyRK+f95R+PGVZyI54ijYugWtooljd1MA+to0DE7dPCjM8Nt9/N/y3H823DnPOJWyhmyxiNU79sEORGFYFixb5Ld0IsGg8Bj0vSzRgquQLLGABOvWbViHancGC5+5FgHFgcMeX/xtuWzh+p/9Du1dFVx2yRdxxcVnwaILpci8sLyIJkVb4U1sKCBHsmnTJs6bgsEgX1QLdBHEg55pWQbefON9JJtaEAiGsPVABu37OxGNJeFICvoHcgypOrr74PMFYDWMh5JoRDAkDJciLm1wzuE5n5XYcBWZ8hUJAT9BOkIHNlKqg1vOaURTywhExhwFywxj6bKlePfdd9FdqMLwxwEDKJbz0EwT08aNxi+u+y40M4CvXPgLZPN5HD0hiZZWP+pSKUhaGU31dVj38VrsTsexZdNmtI1s4Yt64EAHHQRikRjidcPR2DgRDQkL06fGMG5MC1paGtHc3IC/vTofjhlCT08X1m/egZIdQH/GRDCsMtqhTeVXJRBMI5YiHE2hr7sLo0c1YOP6tUzYsHGoAeYi/H4fZNmGKsVx5oP3IkBOLRhAbKAHxw68i5FNCV53XcvjP19ZiONPmoGGuhhOPOdCdGUqGDlsLLLpbmzZ1YXOTAk7uotoVVU0GxvwwdJ1eG/pGkyfNgXRoI8Nlxy1iFoUBhzeD2KPkVEIo5JlkfcyWaXI6BzIoj9fheRYOOWkGXj0rh+jWCrD7w+IvUEGBQeWaaFULonXc0R6d6jhEkT3jJQ+e8fiwXQ6nkAoJN6fSCjbxDeu/QP6SiK/pSAmILcKWSrh+TuvwCmnngwn2gSjXIKpCV6Hoq2XchInQScnzon28cGG6x1DbaStNeyDI+6cFxx6wXw+j1XbPkUBIZiuN6YX9zwhQUpeG9vkjc4naBv81rlcDls3rsG5R4zAb/59JkcpQ5ax89MO3HjLg6jqfui2jnAwgCsuOR0Xff1USGoYNhm4ZUM3CbbQK5Gx+HDf3ffAMmUR9RQFyUQCDY11aGltRENDHSCVGWqt3/AJLKsevkAIn3VkUawa0C0H+zu6caBzAGogiGgsgT3daQSaDkcw1oBgLMS5G0UYiqzkrdldsPHK7HRoC8mSLTavLCNoWbhjZhPaWtsQHX0MNDOMNWvWYM7rc9CercIORkDeqGIUoVdNtDbU475brmMS77SZ98ExMrju+2fh+GmT8Lc334Bsy5wv+n0h7O1K4d0P/go4Oh8T5dm6XmGSLxCIYerkmYDUjWggjRt/+h0E/UFOXwgmd3QeYPZ007Z+PDdnCzLp/TD1XjiWAZvRggk4ClQ5iFPP/A5WLF+EaUcchfXrP4Bl98Mh1FZDhKi06UMxfP+Rp2GnGnlNRvRvw5HlZYgEAwhHVISCIa4weGzvmKMvRFHycVWh78AO9H22ktezq6sH7fv70JctYf2eHDZs3I6Jk8chFgyCAAXBWK5a8FoLR885JuVvFCdti9MYj4El8NrZn0WuojH0v/m67+HbF5yOYqnAzp1gr8cq67qGarUi0JxrIl5kpc3PP6/Jb2ujrWcojDTDIjclY9MNA1/9wf2oaH7QVmXiSZahUOrns7Ds2e+jZdJpUKQQCoUBSA45UMtlpcXL0LWqfdQa7ucZa63RikA4hBCkd9940aGDIGZu+9792J2uIhiNI18sD7JYnD9wDkjQcsg7yQx3KQoDH320HAFNx7Lnr4NlG1i6aCneeH0V8mUdVd1kOFhiRs3Ed751Fi666GsMMYjrEnmKgObLl67EiiUfApbId8jzOZaNUIDIJAXRqA/1jQVEo5R/qEjnYgj6QujOGXh35Qbsbe9DIhLD2LFjEI4nsGnbLhzIO1CSwxCIxBCOBBGJEUnlRzDgd8+JclmBMCjvo+iryjaTPcQkRmQHd3ytwTXcY1Gq+PDJ2rWYM+d1dOU0WMEoHEtCSS/BMYCgLOHxe29lVHD2hQ8iFAihpa6Ec04ehzETJuAvr7yJdRu2wLJUnHHmJZj9+n/CsEqCA6B8T6GNHMDxx50GvZKCjh7kM/tw0w8vwbhxTcTxIxJOoFQsorOrHZt3FfHsnA5kB3bBrB6AY2XhEPPMgddBou4whCPHIp85gKOmTcWqVe/BsnshgQi8Wq9v4oSTvoThF14Ju60VMSqNZbM4r/wGI61EIopwKMjGRAZsWjZGH3UBuopVRPwhdO3ezIbbN9CPnp4+VMsWduzpRE5twOqVqzBlymTEwkE4xH0QQeVufoLSTKR5ZRoi3QjJ1+xmw7LRly8hUypRpQXP/PFOHDd1NEdWMlwRcYVD0DQqRwpy8vMMl1/ZEsTUoaUgj7kleO4nppqDlYWiqeC8q38LnegZm/JziqiCT2gIGnjz6evQNvF0SE4A+VwfVMnPTt/jZWzLYkL3f2O4IuqLGO2t0aDhUk6QzuexcnsHlGCEa4CcIzA8pg1NueAQeUAHRAYlfCYwMNCPLRu34sGffAUL5y3Fkg9XYFxTBD/4xnFQ/SYK2SoyuRIMUwGR180jx+O4U06FYzkwyP4p4beAmd+6FhWNDlCCTBfCshGNRhAKKQiHA8hmswxnJRAEUeD4FZx53CQcNnY8Hn7+TRxx9LEYPXo0ksk6xJIprPxkC95atBZWKI5gJIxwJIJQJIJwNDxouGSoDJU54eJ/8PuEU5HIcCUHv7mgCU2NTYiPPQ7lagCrV63C2++8jfZ0BXYoCttwUHEMmBUTsmXixT/ciXKphPMufwTZHHEGQJiIp7AFxwxCkoKgYF8fj2Lfnq0wtDwzxQ50Jl+IufzmhZdh4/pOpMv7EAr5UBeuw+XfPBqpxggTTMSyU2R55fXVeH89UEjvAcwydG0vR3AyWhkKxk8+DwN5BY6RxfRJh2P5h+8CKMD2nIVrNFSrnDrpTGRDEQw/YwaUxpGYFtfxZX0hfD4LwUAIkbB/kBfQdQvjZnwLOUuGrRnYtGoxunYsh2YYyGULyGbK2LanH+VwK3Zu24wxY0YgFgxAdmwYZAFknLbNXEPtw2aoLwgpLxoaFtBfKCNdKDCBOeeV32FMYx0q1QqCQQ8qi/JMuUxEnyhZ/k8MVxgpQXSZ0yjVI5UcG3MXr8Ksp5eCDNCrnBA/Qsjm3uvPw8wvTUW8ZSpMXYamFSDZxKGI8io9n2yJUqH/qeF6rPY/Ge4/3vxPhyhqgsvFQgGfbN6BPtvHxIa3aH7Fz19zHkJ5oELlIsG6eqUf2ZGxZuVHMHUDl55zLK6//EuM9Z1KN6qVKtKZNDID/TCrZfhVGUEiqIJRjD3meE726QA7duzGe6+/jkJRh6P4YYrsBrFoDMlEGLG6FJcT6PndPR0wDBnwJ5Cqi0GzVVSUKKKJBLPb4Vic2dLO3jR+9/SbgD8GNUL5bQzhWAThcMhllVXOuchz0jlRfsvVJoYmJp9zQJVw/8wWNDQ0InbYsdCrYaxavQJz352HfdkcDH8CtmGjajswqzpM28LLv/8115Kv+dmz2LSryMgkEkkg6Bfwj6KN6iM0YbIoISL72UkRdFdhcU5HHrp3YACSkub6X110AlQqwTJBSLyAhWRdmNnskjQM7fu3wC8XUCz0wrAKgK2zcGD4hLNRzNporIsjEVexaeMKhEMqKtVuEKwUD4KpKUyfei62bfsQM0b146YbLkYIKnxKnllbZuOJA3DJvELFwLgTr0C2VOVIt/wfrzGZVs7mkS1W0NWZRY8RQFaz0NXVh/EjmxFWVdiwYGhVvrYE+wXxKQzGE+uw3brf0/OqDtCbLqJUIi2BhGX/eAqRoALbMvm6kQPgNbFtlIqFQeKJN6kLj5l7oW9Z3OOWgtiwDgaq9BpUzQAhH0eBQSjxlqexp6sA2ySRzJABUgBe/vSPMGriZCjRNujEJrvkFeXe9CAcRdeb7clNTQQpO0QO1gCfwYMZKgV5PyI7ETm39ObsFxyCFSRWoGL+nvZubOvsgy2LNyXoKFFdlxhPiS4veUg/wxOCuLTZaAMR2bBl4yZolSoOqwvhtSdvhc8JsKF7LBoLZajUxAdNsMHi8o1eLsImn0BMo15BVTNQqlSYVKGLwlAl24mBgQHEQn7s7yshFG+CpgbQnzagBMjRCOaRVCrJVB0Un8rOiC7nDb9+FAgm4YvEEXYNl45fCC9UdiSKsF4mSjzhCUt7HKrrAg98vQ0tra2IjTkWphHC0qULMX/+BziQLUL3JWCbNsqmBVMTkeT5+38JvZLFc68sxe+feBeRSJyFDcKLEyynPFeFY5oIKn6komHOa5nIcCReg3JFY9hnoxO6pqOx8XD4fZQH+/nYy2XaNhZylSL8yeEY2SzhxceuRkXTUSxXUK7o+GxnN+56aCkG0n2ApaM+kYJjlZmIAqqQ5Cp8ATp1A4rUBFluxuYt7+DbX6jD5ecfjkgsCVkRiEt4NPcYAZR1C2OPvwIV00KxVMLcv7+AysBeFHI5FEoauruzqATq0ZMrsUOvT0QQpCgrO7BIrOJCR495ZUEEGZXjCHRHXArVYh0gW60inaf10LnKsXzuU7BM4gmEIkkwWsII8/ksfy/qwHSeLpHkGS7tWfd9DjZZfia/XiQcgUOGa0msirrkhkexr6cAIgYIGXqQmljy95+5EiMmnQpHjaCSyUNxlYB0DuyU4HD9VhyPeLBRDuLVQYL/0MNhJOgFULZHlx2X5rz6rENJM21yqn3mixUsWbcZlhzgheMnkkzQ3VSkcmEP5zgI+Ag2CW9JBrLr08/Q19OLsKNh5euPspqEuTPXy8jMwokDIWN0qKxNTsiWUJUcKJTbUCQmL6dbkH0+UViXJQSkAG6+6UZU8n24+LqfoOyQ2siBZDgwbR2VquYSHvQ3VI8G18wIkl13+28hh+rhT9QzxR8Mhxl+E5PKG4QgJW1OVomJTcPHLAlYpCoSfvf1VrS0CXLKskJYsngB3ps/HwcyZZihOi4BlHQTJknaHAe/vvZyjGprwPtLV2Pb7j5YpgPTcGCYFtIDWVTKOspGGZV8EX1d/ahLtXA9WcBHKtTTcx3ouoJYjMwzj0J+AKbhhyrH4Q/4och+2I4BWY1AbRiLpoiMvz75HT7eQECFLSnY9lka37thDnp79wOWiZCa4DTAz+UuujwCTdF7F/ImLFTRn/kYt1w0Aqee0IAEIRN/lEk7TmBk4jkEE7+/ewDTz7oWhaoBzaji5T/9AXapm6FqNl9BoWgiMmoSPtm8BZFgCFFFRpA2L103xxICCTcKUTpWy6p6m5UdmSQhU65iIEdSR4ed96I3/4iqriMYoDx0yHDpNSnieqUhQlK8prT3aiIuMc+f9/AMNxqNCqEk1YR1BZfd+Ai6shoss8yyXK+Oe1hLEK88eDlaJ30Ztiyjmi1wGsOkrquWMmxxrrXB/X9iuJ6he8fL8Pmtvz7mFHUHFc1EqVLm+tf6rbvQm69A9gVJzsIqHM5xVSFpZBgj0cUX5RQhxwJKxRK2bNkCx6jg2m+cjqu/PZNPwjPcIY9BjsuVmx2iYZZJ10nqIVa2uAbEb+hg9it/weN/fh533XcHjNgw2FSy4ryBlFyibkwPikZ0POSMtGoVT7/4KjbsLiLUkEQ0HkcoHkUoFB6MuMIjk6xTASlj6WvWzhJ5IQE+MtyZrWhqbER8wrHQ9QhWLF+MeXPfxd68ATuQYqOoUv1OE6TI+eecgW+ccQIKpSzLIelBx0JsOCl9mEF164tk6PRG9Ds6hXSuhFKxikymhP4BjevDp37xSPiUMhzbh3S6jIFsDh3tnejv70P7gQFkzDZEI3EMawghlYrA55PR2tKCiqni/cW96O7fCccwkAin4AuG4VcDzHIqfhlUDqRlLJd02DCRL27AQz8cj+mHUXpBjs67znSph67JrgM5TD/vGlimjWK+hNee+T0qxQFUqhbGTjsOXekqetJpLFm0GI119fCTcyZqjYVvQ/VMj3xhYyAipiYaUpAgdplUcgPFCkzHxsjmFN565bfQqkRaimqHZ+gkIS2XCoKpGvy5iHOsU2YbJ2XfwfmmZxQE+Wn/hUOkUVZgwkBH1wB+ePdsRnwCFVD1wWTE9Kurzsa3LzkewcYj4FRMvsYsgXRhMr2up0/mczvIWwwRg14Er/31obXbg3732aLHnb29Rezut3njFasV7GvvwNbdnZB8IRH1fKqraiHjpbrVkKqKYJuAKiKSbt68GVqpiIRcxtI5f+Z8YjDiuh5ILKJQYnkP78AlRXj0SqWKUHCoAE7L/OnmDdj+2R441QxajjyDYTY7VFcaR8ZApI4HgzivIK1y1wDuefSvCDc0ItXUiGA0zLU/IXEUOS0bK0dfCSrLBQnKCKilysAD5zWjrbUZ0XFHo1oNY/VHy/DevHnYla5CitTD0nQm2ei4CU20pSK49Yff4U0fDoawa+dOTJgwwd1gYv2IlffIBzoILoPQktimEMEwkqE6pMzFe8OgRg+dy0UiehuiZpnpQX9/Gc+9uQ29OQOmYXGEN9xIWjUIHSXQ17MTjlNAkIxXjUCrUp5HJQoiIKmgI0NS/SiV9uDF20/D+NFJ2E4RPjkoUiZeZ8GU0rGtWLMbX/nBr/jY8tk83n71JYwdfxiUUAP2dvShK92DXN8AlixchGQiCR81oxCooLV2RRdebuvVT739MFjjddFPX7aM/nyJhUGXnv8V3HzdRdCqGsKhgGhIcAk24lM0rcycRa3hivRMyA5rm14OsiMBqhmxEdcgCmoGlq3Zitsee4+5Gk4XmVC2+PfL/3Ijho2bBCXQBD2X5+OgaxIIR8RLu6UkjiT/pE8eMtxDj8OzGc5na0p23jlJBz563jF1DX35Cj7emUah6iCdyWL+ivUccYPRCBM0JLimjU1Cf853yB+RMscnch6XHUdXVxf6OjqhOCbef+5OJBNDxudBB2G4Q5GYWEQG0czqEsRwFVI1EZeEGUYpi83bd2Dz8vcx6ezLYHXUJFMAACAASURBVPBJUQRwSTJaJK/7ggorlMsYJgbyBfzi3mcRbx2OaF2Kz4maC7zcypPZ0XmyGGDw/BQu0RCsu/9rTRg9ciRCY46EpoU54r4/fz72EHwKJOAYJkxHZpaXan7JgIQ/zroVlmPAJ5G4YUhg4F0kigCs2GLn4fHzDovumRxwyJS5rUUoXQm9sEMhdyK6ZugfEWoWlW4klXQg/HeGabNm2zaqLM4nKSqRYNVSFoZEsLiC9EAOezu6kM0UOOqWKsQtqKhWC/jWKXG8P+99zDh6HGZMG80IhYT8JjU60DEDWPnxAZx79W0swunuzaC/vweFqo5cOodcMY2O9g6EQ1H85aWX0NjQCNU2IdN6knF45Tc6drd6QYdeK4Qg02NVFEHlos51XEcGXnriARw5vomjG9dwXcUUfSaexrJ0l032IrFbu/1vGq7fJ8qEkC2YtoSb73oKyzb3uVSpyzzDZqJxyTM/RPO00yHbPpQyGVfCiaGI6xmue9H/VcT9rwyXt8AhjQdS18fPObRYtOGrpo+VL5v3prFu2y7s39cH+AMIx2MsESTjJT0sRWF6iIglDI2pcdvi1/ls+6dQZRU/vexMXPJ1OinKlwnGDhmrp0cm+BFPJoSHYwvyNjA1wAgWTexFyqJlzJ07B5n2Tkw45Rw4VhimQmSGDcu9eBRlCS6JPFo0O1DB/me/fBRGOIamEcMQikcQcoUMg4ZDqQBLHsWmFBFRgiXb3NJ298xWjB09AuEx01GtBLB6xVLMmzcXOzMGrHAKEhFTJCYheK5pXPp56r5bQfXH715/G0cs4glCQT87wNbWZoxoSDDhNXrkKIwZ2YqoP8A1cDIM3ZLhc0j2Jwg6Ph9Sj7kX0HbIcAf7MYauO62fJNaktsBPZQvO+zjrcL04i23JH4jfkbabriWhDSLk6BpRC55qmUyO5fJZVKv9qGplDPQPoFx2cNzZX2NisrtvAPs7u1Es6yiVirh71p24+qrvQfUF8ecn/oTmVAphejOviUWRmARkVEHOyJXUkiKJzlE0CIhcmn6fq5jozeYhOwoWvfkEEhH6W2ouoDyf64lMDlCLH8Nk9yJSXsuojzMqcf619dta4sczEHLqvC9ISGRZOOfKXyNTFRGU9xqhMBs48eiRePRX30DzmJPZWZZzOf47Nno3paS9eBCa+Dz6mI/YhfPu9R00VBdJ/JPh9qx9zuFNQR+mwdEiW5Tw8ltLMHflTij+CKYeMRWf7t7JjCiRIvFEwu388fpYRZMAlQmohW/7th1wDBtNEQPzXvoDQyPR4TDkOTyIS9G2kM8jmUzyoVMOzZSW46CQLyIeF0JvWi5SAX3w/tuIROphGjpCreNgugw7HT/lJ/T+XnGcFo3E9ER0zfr9k+gqSmgaORzxVJKZcc9ZeGQURVeVWC3PcCUZlmTB7zi4a2YLRo9oRZSaDMoBrFy2CMuWLsG2vhLscB1V/hmmizyWmiscPP+72/nrS39yp7thCaEIpRZvGHdN6Ou2hA8NkoWpk4dh1cZdWLlhL8PJUDiCYCiISCSKRDSIQCCIRDyBpsYYhg1r4xbG1sYGpJJ13FssSSoz5HTuEtUy3dqhR76xQTuUR4quE2om4fXmHlEPFdB5O1AcarhQBGHIcJqgtIyqVmFij6A2VBO2IWNfVxe6+tP4aNUneO312bANDTffdBP6+3vx1OOPY1hTI/ykTnG9DfEGQn0lHlTjpPIdOW4my0g1xShMkIx9uQryFdGK+MmilyGZFShqDVJhMYWNfD7nGq0LlV3iiq6HMLyDO4J4b7lr5BkHrTedK4lhDEvGGd+dhXKV0Jd4DVuiNhsVd/zwbFx20ZkIN4yFSalShbgCWxBmruGSymwI9oqU8vOgb609H8QJHWLQ3jlI3Wufc1jVQUl9tYJqoYRyWYM/FMK2/Xk89dpyDBQM9pWkJgmwiCHMOk7aeNSWJgQMChe96U07O3tQGMjCp1pY8Oz9iEXpovs5EngH5RkuEyQ2XRyDI5JFulmfn3Nq5ni9xaJo4/jQ3bkX/fkydm9ajZYjzxyMtMK43UK3y1YK2EzG6+D1eQuxYOVOJFuaUNfUyAV20pF6UkfBIjtsuF7E5RYz2YbPtnDXzFa0NjcgNeE4VCp+LF0wHx9/vAbb+8qoqFGGoQTNqfZaJYG76eCZ+3/O8r6LfnzbIISSub9TkGEE8/lC2DaSYRWtsoEjp47Avo5+zFmynZ0T9YN6qICCKUUkyqGI9PM0s9Tw7UUpLyrQavgUkatFImE0NqQYriYScSSjIaTqUtxumYzFEIvFOHWIxeO8JtTU4VeE9JMdEkdwj+Bh+o6dA8H1bDqNluYWbPp0N554+jms3bAJDl1Ho4o7br8N27ZswquvvIyWBNXgqZ9Y1GoDPoEk+HjdmjStH7XwCQZYlCJFLyzQNZBHUTOYEP1o/vOQjLLYI16KQa2mBkX7koAKnsqo1nBrIm4tS1RruLSOdP7CoE109ORx/o1PcJ3eg/EWCBWpWP7cjzFuygxYviiMcoEbTTyZI+nl6UFk72AmSzmuLerTtQ/vfL2f/bcMd/+KPxEi4YdR1bFly3a8N28Bxo87DKPHjMawMRPw47teQqYE7vUkqSCdGBluMBxhY5aIbeacC5xzkLpp3/79fMA/Ou9YXHX5RXxBFDrhWqxu2kxsMJqxLCa+iBn2hyJQqNRUU+fyOEASDGzctAlrly3BUedezJMRmMgRtQpeOIKqBJmZpLIZ2GAgncGvH/pPxBobkWhqYQEGl7gIiioSZJUWlcK38PIcDchIZBM+W8JdRE61tSA1fgZKZRnL3p+LVavXYvuABiuU4IkOTAgZhhg4YFl4bNYtUEwDt9z3Z/RkM5AUHxziCwjNUsC1BFtvwIRP0jCtPogjp4xGb7aC5978EJIpwxcQm5PzYArBlN9S1CASjjeX2OS80VwJn5fzeaQdfab+Vc6YiQ+QHS7JGIZGrS01yjgfrx0Zu991xuxguEtM9GgHaQiBP4D6ZB3O+9oX8bVzzuXOrY/WbMQtd97HnUiU85KTvv7a72HHp9vw1uzZaEs1MO/Bx2I7/Pqe06RrRpvZg5W1ZKYjK9AtG129GU47Rgxvxtt/+Q0qJSAW9rP80/V+zN6S4bLc09Wcc7p1SOViMBi4TfC1RkTOgpvyGShLeOHV9/Gn11cy289+jI6VCSwdq1/5ORomnspcTyWbHyTwWPOgqLy3KXhw6Yd18Ac3FXhOdojfGGLHBc8zdGR8LWt+IA1seM5hNlbXUcxX8MxTL6OxoRnDRo/EmLZhqGuIY9GmDtz3xDuQFIJGAi4TbCZZoUyazlCAWUm6EMzYOQ727t3LTm101MHsJ+8REccRF0hAWfrWRrlY4uhBzoCen8lkEIklEIxEWEzheUPKYfkhAYvnz0NfxwFMOfVcFCkMeVDfERCRPjzDJa9Ji05tgNf/8hFE6pvQMKwN4UgMikr5uegM8vJIoVl2F4zgNxmu5eCu81oxavQIxMYdDa2iYvG8d/HhilXY3l+BE61zZXyUU5vCcG0Hs356FUa3NOOPL8/BstWrYMsqVEtlgo9guUGmJ6vQTAthWcdRDXFMmDiCHeRDz/+Dtdgh0vZSzsk1bTFKiNIL2XZQJa0vORzSWrmdVmy07ugfzyD4Z27nDDszlrDSMAoS0IhrQamDQQKYwcYSV3BB6YtM4htBlDGh5xKTV1xyAa64+Js8fGDhh6sx68E/uq14JGJx8Iv/uBaLFy7C/LlzUReOIEC6c76MDqgRj5w+oQeueXKaReIGKsWJJhbarDROSTMsdPWmWc134vHT8dSD16NUMhBx94zYFg5LTNlQXMP1Jmx4hisMxW2i9wQbNVZL78f1cR5mQCN1HPz0zpexbEs7p5GDdWbLxtknjsHDv/wWkqNPZMKwSow3iXWIq3GlkGS4hMC8CHuIQGvwnQ8yyEMY5IOjMPE2LvLJbX2BySnabO+8+Q5UuQ51qTo0NNbDFwpg82cHcP8zc1G1FDhU5yRvTOof9kwRhBMxzsHIyOgARA0W6O7u5oVsifrw9K+u5KjI9UNipSUgGo3xpIlqucJCDhLMMyFB+YbqQyQaRyQWH4zQg4YLB8uWLMa6lcsx4+RTobSOdw2XAyRffJ6+4ZJUJPRnHbRZxX/85gk4RFANH44wvb9LFFHvKpdEXEb7nwzXBu76agtGjhmBxPhjoFf9WPju21i9ai229pdhBOJQJUIPYjIIQWXdsPGTb38dMyaPRyZbQUNTM9K9adh5TdSMKSKo1DoWgOyXIUdCiPooT7aglUrY2UNCBgtVU6AHypUo18vl85xH9/TleLJEe0+/iMLcpO2q0hiSDbW4MZrynCVbjnAAzE37RF02m80w++1FQYLBXjeKKgvikDckOW8yLknCz677ASaMaMPEw8finQUf4uGnX4SP5bEW/LKD6665DCsWLMHyZUsQ9QX4fD1HEXAFCpSymIYQt3qkIh2PcPBMx6GiG+jtz3EU+/bFM3HzNTNR1g0WdXgEHO2bcqkoXqPGcAUUo2d5wp/Pr9+y8R9quKaG83/0IPZnqCwn1pgexN4/8ZuLcNYpM6A2jGGZq1UlfbkhpJL0jrKCSrksGHhP5lgb2mu+/l8Zbn778w7pL++5/wW8/e4KDBsxAsNHDceo4cNxoLMf+3uK2NbeCVtW+KIodAFcrSoVmSPxGM9v8gfDorOGk3qHHUFPdzeSQQkfPHsPbMliVRItABmKbFqsaiKpXDAYQi6bY8KDapBkzOTZQ3XxQXKKYBLlN8Qi9nbux89vuRNnnDAV4864EIZFr0ksJHlKmwk2ryzkko28TE+/8Ddsas+jeVgbQvEEvx9BP4uQgNuT662ngDZMSPLgr/vPH4GRo4YhMeEYWEYY8956Ax+vXoGt3QbMcCM3mlN5SjZp7EwVti5h5qnH4vvnX4AVb6yAUwoCVZlzZtpcZCB0Tixo55IHnR8RQRThCOoR/Ddg+2zOP4WWmPo7FQSDVJ5z4A8HEIyFEUiFsD+Txe33PIS8prNEj6SlXFvnHI+rbKJBnZwas/Ui33JkEdm8/lJO9bnrRaAdzxnTurBTptKd4/Da3XHzDTj6iIkMHd+evwRP/OVVhtMUxJsSUXz11OlY+/HH2LB2PYJcTpShGzpHVR/X60UE95AaiVeYnPTQFaVQZABVA725PA8l/OOsn+L0Lxwp8uRAYIgDsSwUC0U3PxZSVeq59R4eKTXYDcQ0sxuBuaVU5J5iOJxIOyi9+MJl93KrKOfhruHSMS5+7mqMnzIDUrAeWqHE50TP4sDE7fsSpx2i1Hew0MJzEt7hfR6z/S9sfPDHUvXT55y5763Ev9/2AoupKUeh1q2pkw9HS0s90vkC1mzeD43ADeWDPClClDaUQICVSKQLDoQifNG8aXZ0pvv374Nk6Vjy1z8ipGgiMfdOQhKb1svHPAhAhMoQC1fjHW1R5qHSzorly3Hdzb/FT751Oo6d+R2Y/DomLEkIKMhw6XUJ/hNbyR0dkoRVn2zCy2+vQF1bC5INjbzIPJrHJ5RankzNg3MEKemYKZreM3MYWtqa0DjpOJhGBAvmvoOVHy7Fp/02KoEUyztpjpJtUS23jEkjm3HzpZdh3RvbAY2YclETpjYh0oYzqefIfHykt5Vk6h7REQ7T0DOFCTUOiyYpcUSDB8kYaepAMhV1yxIWSw2jagRGtIopZxyFWY8/g4+27WSBfG03CoEKWj/elK7x0eant6G1EnBSEEJ8XWzRTMAbj8tFYs8QLPSuz32/+jnK2T5MnTIZr89diL+/+wEjCVru8SNacfnXT8Pzz7yET7dtd6cdSowcOGq5wgpKkYiNp23BbLw0NErHF6TyGJAt0IA9mthoYuHrT6AhKdrtvPRGnJOFQp5KQaJ0WGu43kA4z0AEXBaKO36+a7i0CNFIlH9GFQq6Zid88ze8LqTY8gw97lex5C8/Qtv40+D4fKikxXyp2mkX5JQ5fXHX1tM+1BqpZ7i15NihxNW/MmBp2Su3OFde9yDyGimEZCYe2lobcMrRk3iwmq364QvH8dr7a9BbKHGbmOclZV+Ap0n4AoIkYMKHciDyzI6Dgf5+lkGed8LhuO36K+AjscQgoyY2iPA+okDueSLvYD3HK57nMXE22tv34BvfvAbTx7Xhmlt+BZ17dkm44P6lI+qAJOwW8Fv0QqYzRcx69BWE6+rRNLyNaXuewkc1atfzC9gp4JXQVVPwMznitrQ2oXHKcTC1MFYuXYxFC+ZhR7+Dii/J4nMGfJaEEfUR3Pbti/HRq7tgFkUOGQj6xEhP+nAlo0Q8eudNAwQo76Q6L11sPmYaWkDjarlPlyZOAtEYjZMFR1yCspSn+ijXI8Y1KWPy2VPx7VvvwYBG8sCh+UbE6guyina5KMsI4cOQ4MTLY4XAwpW2shELldbQtRLr/PA9v0ZDjByNjRf+/hYWrFrLLXqaZmHG1HE4dnwTZv99Dtr3HWBDpbDvGS5BbZYzqpRiiYkSwjG7cJRQCKES20auUEKupENyNHyy6BVItu6W1Ya2NeWTNCBOMLT/O8Ol4yFy1TPcVWs34fr732HeghpYvP35hSOH47l7L0F8xKlcS9bpfWlAn6dFIHmrSeo1IumGorln+IP72/3if2W4k+plJ1bXgC9+4Rg4RgnTp00k14yq6SBXtWlOAwb6s+guaDyKdOeefWxwXLLx+ZmcolojDdCicgIzj/4Q1wdtW0NfewciUgVvPv8gE0FM8HMvgVvXPUQV4m0e3l9eXZFgGsE+0gvQTCgHWLhkCSKxJvitPIxYC0945KYFd6Eo36CckDuEXM9Hxv+TXzwEX2Mbho8YjmA4yOdBPoGIEq/vWLDUohyiSQ58hom7LzoMI5rqUTftJOiVANZ+9BEWzn8T2/pMlH0pvgQ0toZkfU/+8iZ8/NxWaBoxzIQ0bC6zcOSndjIvV/IJFpfbJCUbdXV17pwkMQ1C6GIN1j+LlkMH8XgMlk11VAWBEMEym6NDPBbj802NjmDBgd14fv57sG0xVpSWmssr7tpQV5qAx+I9BvNaYtTd60ENDExCsx5UuDF+rivYp/N9+sFZcHSaNAG8+tpbkEJ+TrF6OjswvDGJpvoEfn//b5FnKEkbW+FZw/Q63JVFY13IoN3ha8KovZxQ1JlpDwxkcihrxIWo+Gj+02wQYkqlkImSsWpahT9c6onhA0NlrwTEsF8Qp0OBwav1iqBAxBR1X9GDHP3jL76J1xbsQKFcAKwAbNlkNv61h67FscdMgD85Fk5Fh6bTNXZ4TJD30Fwya8i1eNLcg37C3zDicaW7tbCaf1ejiqwNbtKcP1ztkGiaCu0GVNauHujoga7ZKJky9nb2oaw7rKSq2DTWRjBn9EGGq6gBxIJ+qEEFpxw1FVde+k2ESSjg2AhbNBhbiMp9chWmFOA+U8mnwMewzGVwCeKSQoa6gOhCuJGBUz3RwgKLSjMUIcgzWxYWLFqAYWOmYNeH8zDsuLOhSTSYusYDmyayuRzDZc9Tkme/7Z4nUA7GMWLkaFAHCJezaLIjf/YQgDsilORq1MZoO7j3orFoa0iiftoXYBphrF25EgveewObe6ooqUneQCSPu/obZyHVIyP7qYlSucqCAsMUxkuOiyINPTjHNbwoJiEeCXInlBeNvc1D5JpHuCXjMU4JyJ0GAz6efEnMeLVSQoqN3kSmUsLEfzsa377pTuhOCTppi60AoBK7Keqi7nivwfzVy8Pcyq1YRMo/XRGBt6qsK3bHzNC1ePHRB2BrJRSLZWzftBWG5GDNqtVYvGQRfnv3HQgHZNx5xywUCmVGNz6/yoorehApRVM0BFkl1EZUyqFUyHuwZlxR0dPXD003MWXiSLz69F3Mi4TDBGlpWJs324wcgilKYm4XEIsuXMOlTb9h/TpMm3bEQWUVNg4XzRGxJMnuPClbwm33PI61e3X0pwfAzs6h62di9as3oXX8VEi+ZlRI8OEesme4jPZchOIZJn3mFKTWbt0KL5eL3K//leHWlvj4er36++87FhtjgJVi5Dn27e6AIUnoyVXQmymhL51Dpmqhq68Cw5U4EsQhsqohGcEDt/07Jg9vwd63lwArt8Ha1wt/XueezwANOKeD9lE+R80lshj9SkO8KJ+iIrwfMGmjBP2QkwnIflUoelQHKs2Goo9kDJFTj4D/xEkw+srYsHktwnWjsP69VzDpnEsZFnq5G60NeW+PiRWmT9vDwux5q/Hemk1oGzGKFUgEjRSfYDC9uVre2tJikkMIeIbbmELd1BNg6mFs/PhjLHhvDnamHfRVfUKcDgOP3HwjPvnLVlRKVGKzWMNt2SROFwNzPWUWXUSv3jxy5EhUCrlBgTvls94xm6YYek5N/HpViOdlVTjPaJTywypSdcnBUgV1Ek09ZxLmrpiD9dv3Y8n2PiarPJKJ2dqaAfRetBUbuGYSBXEQg/ppsSJkFKyTdpveX/rjA7D1Mk+szAwMoKOrk88zFg6jpS4KSyvil7fP4rtJ0GtRbu85K1p3ym+pU4rgMR0Hiyeo1cF1oMQ/6DbQl0nD0B185/Kv4hfXfpMHG0YOMdx8ITvUEfQvDJfSD683t9Z+PMOlVk8aLEc5r20pePiZv2Lemg4eAqFTSc5S0NIUxBtPXoPh40+GLIdRztH7esMlxFBFRnsui+8FDe/9/p8Z7uyHrnXIQ9BG4EWVVOzZdwCmRcJuDbmygWLFRJpu79GZRbEsBpEFVBUTxw7HCw/fgX1Pv4ny3xahmVhTy4JORjkIwQTsYxKopuOfvCNdZN44rs5YnKSASsK7C29Kt5fgMpSiwnfTv+HTrn6EfQ4yMw5D+7r1GDZlBhNUVCIgppE2vUZif53GwIioxqUMy0KuVMHb7y+FJgW4XzUQDKNAYgYSRih+FsE7sg+qTBuUDIhezcZvvzkWTfVRNE05EbZUh/WrV2DJe+8gmQihLpnk3tipRx2PHSvzyO2qwqLSEOU5VCs1RR5JkNbP6guX3TVNtLQ0CSTh2Oxo+JYo7JldNVu5xHJH2uRapcxaZuqljYSo3kjGX0HbyGZRBnFhV3B4ECt2LcTuvQfwzpo96Ncs+AjNhEOIRxJC8caQkGCP28pI8kFXqebVK72OILIjFnCwkIPKLQ6CqowXH3mAO2b6+vtQyOYRjkaQyWZQLlcxpq0J+YF2/OK2X0ORKbISchDQnPy2SlDf7+e/p3Wn1ITOn3N5cuZUEqJJoLaEvv40qo6DR2b9BF8+7Rh2eMGggMrMHtLAwkKW0wbBJAvz8FhxL+p58s9ao6WrSyiSrg8TU44Kw67wbO47H/or2vsr2LW/B5aj8nD1S75yLG7/0SmoG3MG5+Ua1W9twfyzU3RJtiFmXPSY/1cPdqo1TvJfTcPwXoMj7mtkuG4uyPS17EOpoqE/W4AkB1Ck5vqSxl0fNB7m48274TgBtKYCeOflx7Duhvswav2AgIPEvhEb546uZKke3cbD1aSqzpDQgVQ7NNWQ8z2X5fS8E0FKEmnwybh9v2yQkoRqQxSNc+7GppN/BPX2i4Axw5Hfvxtm8yguVYjiuchnaCN4zdqstWV9LDD71ddw5umn8t0HaPRJKOjjMo1m0R0GDOzsSGPSxAmY++EaaHKUZr3jwUsnobkuiuYpJ8FEEhvWrMSKRfMR9pNEzo94LIkTjzsHi17cDVu3eRC7ZwB0dwOumxKB4U7tp6maw0eMEPCONrM7eYGcZ5SYZWKp3aFq3NRNqYJOUjtKFQzWLVO0bWigCRWWmG9EghFqUE/5YLSZWL1yKd5euA4b9w3wZPdwUMW3vnwKlrz7Ks784pfwyYEBZKsO9FAYCo0gqelh5fUSN1Pi82eGlCWJVHqTEPH78Owf7uc17unpYeecLxTQ1d2Nhx55BM/+6VHk+vbhF7feCdumqZQElwNsUrTfAm5XD527lyKwcMaVzYpyM017BPr6M5xivf7sA5h8+HCXlRe3BiGWm4cdVopC6+TCYxaqHHrLm8EykyjveA9voiRBd3pNmvl1oL0X9z35Jj7d14dcmaoT1J0r49kHvoPTTjwCgYYpMGhyC6Eq13Dp9Qi91g49F4TgP5eDatllrmbUPudz8tpDI7f0/KzLxSBb1iJTKUblG2gRPCYIoWkmjwwp6TqyeQ37enqQyxmY/dxDwOLVCPz5A5gEAWkEDTUp0NhN13N7hjsoYXNv6ET9jjwS1VXI0KoMlYAczjW5W4T6GrmGKYkB5pA5V4r+6UbseOlNZHr7EPjFldi//D00nXAW3yFALIjDBundqMzzvASVaNPdcsvPccIJx2PSpMPF/Ct/kEtgsWgQYWJ/HQV2tYiySZMdbGanT5/Wgrpk3DXcBDas+Qhrli/CivXb4Jg6vnPxZbD3R5DeJ6Zc8M3PPPUPRXSXLaVxK4Q+6urrheCdWt34njlDk0VMQ0MoFEChkEddHT1PRBVTozUTs7CIzIKkI5GMIOgXih+WDdo+FJw8Wk9qwfxF89DbX8Vjf5mHlrY6nHPSDMx56SWG64c3xlDvDyHZ1gC1uQmfFVR8mqEZxUIn7m0URkS0nu45UeHMr0i47gdX47ipdFcGEz09vdi1ZzdHm/vuvZcVXS8/+yTSvfvwy9tmQYy1IqcllHVkoH6/mJfNyIxHBymMSLgk5DLZPAbVtJGjMo9s4aN5LyEcIsmoGBzvGS7fQ6laEvk3BQ33TgS1UY73xb8wXO6G4vsECRRChjd37hK8OG8j9nVmeFwxlaLojhMfzv4ZRh52JJxQGyoDNClTnINXU6Zq7v8Xw33lge+x4Yq8hXprxaym3nQO5SqVJGQUylWkswXIaoA1t+OGjcANV16GjsvvR7RiQyGFC3kaunuBIyLloMzLrft5bCVtANq4NLOYWU0yWpe1pIgkanOiBhbwk5TSHSlDdxzg+wYpSI9MYuLDt2Ddt29F7398Ax2fzMek2LoysAAAIABJREFUf7uKo43nyUhKRyIQik7UIUQRi2vQEnDnXb9DV15HXVMTR8CGRAz18SCSYYVvp0JN33UN9UiFowjTqBufgekTGpGIh9B8xMmw7QQ2rluDNSsXY9G6nShYPjzz61ux7m/dKBXLyJDTc7tQ2Ou7JVkel2LbSKXqWHBBtURyWNyd5IjeUxHZ6H44VdTVpcRgM3dig2hXFvmqblSQSoTgUwzWM5N6jYYDyLaN3lIZU86fgtmvv4RSuYx0sYot6z/D5s072KHQrVbaImGMTcV4cuaxXzoV7819F62NIxBuGY0NPT1or1AUUOD4ZKh0fUg3yt1TfvzsB5cj6VMwceokVj319vUxYqVzpTbNx558Cj+/+QYM9O3HnXfcC10n0YmQ/nksNZ83OW5XhEIbn/6eBBqeSILSpnK1yudAfMmmxX/lu2IQt1JL4hBTTQ0G5JQFiVMjruD+X1doUSv+rY24js2pCDsPEn0YOq6//XGs20OTN0WLKBXkaDTQ/Jd+hpbDz2SupjxAY3CH6rfEy/C0i0Nu3FVLDR+EAtzIKhx3zQG5XWMC4g9pGWoHWEh/++1VDrfEmeT5qa7mZ8Pt6s1y5KAhbDQXuT+b45IPlQN+c/vt2HjHn9DywU6YpHnlOaokCxNpB99gxKt7eY3i3GcpciVSp4joKHILL+IO1hm5Id5AmObluvI3rrdS2YRQgQ00Ln4YC069CvPVAdjTG3Hh1TdCc6EdvTcZiSB/dJEHsXqI2GMHn2zYiuf/PhfR+ibEUg2CuabJiQrBOIdvSiXRBShloCgmjhnbgu9fdBbqUjE0H3ESbDuJjevXYM2Kxfh0XzdOO/NsNJfqkN6pIJ8roFwSrX2skHLvS8T5tmEgHokxk025aTIZ5+dwq5/bZsdyTa2M+oY6Lp2EgwICewIVT95I+W00TPet0aD6RcSgzRcJBtGRLmL6t6bjuRcfxrixI3HLLb+FZft5YgjladFQGHU+H844+WjUtdRjf1c7OnbvQ8L2s6abjC+YiOPEiy7Gg6/MQzAURdhvY1RbIy788uloqY9C8ScwbORoXlO63SfZBMP8aASf7dzNDrF/oBsPP/QIHJvu9Eh3InRvRObuUS+F4uvqTj6hurSQPorNpBni9qWQqti46G9s2AG/qLXSg9YhmyVmlyg3t7zDrYuuJfDGHyrBHZpriroveE9yDm8RJ2Pi4usfxq7OLAcOErLQq/3HFWfh6kvP4NuMUJ+uWaSJk2Ltee9SfuuKfw5ihz8naWUU+N8w3EHKuqb1mt/v5fu+6/BoSy5TUKRUeeGyuQqqVBCn4rthIpMvolQ1MXnSWJzzxTORu+Be+Gn2DhkJyfP4s3gb2k6DD8/w3FGuRDTxIGxvzpNruLzQrsaWNi+RNNQB4w2sE2NT6bYaVHpSoc76Hna/+yFy23aj9ZEfYv3WPWgdNmJwSh95cjYe8uDuhAUSB5BEngaSjB03fLB5W6ObSeUK6M6W0NWdRldfBnu7+pGvVvkeMOefNAbnHjMKsViYDde04ti2eT1Wf7gIAUfCzAvOx5IX9kIrUBsXOQshuqCITw/asMSYUjtkJBgWEZSaHywDca59i6Mi50kbNx4VZZ5KpczrRPCVmFeqkVPkoteiOzqQzFNyKpAUMaKUcmES3g+UTEyaOQVXXn0F7rj1CqSifnSmy5g7bzXmv7+SeYgff/+7aO/eyY6G4N7WjVuRCIYRsiU0NTdg5NGHY/WWTxGoH43DRzYhEbIQRBWth02H7I/yPXubxxzG150MlwYIUB6bzmQwefIkrF+/ETt3bscbc+YMGi6thefQyWF7hjuIOujKMMnmZm+OhAoNNzctHHf8EXjmtz/jyZWkba9FdMQXsO/9XxouGSbde5mOg27fSRNGv/6jPyBfpuFwpA2gY7Uw+/fX4Jijj0CgfiLKxPBXqTQ3ZLgUlYX665Ce2/+HhkuWRXeZlF598FpupKc3oy4M2lQ0y4dCfpXuuseEEzGeOuh2nHfedgc+/vHvkPz4AE8CIHtj76HSd7X26pIbjsxMH32QekbIzWjciuhYGRwOxtIzMUCO2GfOrWoWgEem0hj0ACm5AnDO/wKkyeOw91ePY/z8h7Fk3SdIJhvEAdAxU47Jt9uk+7WIIWRC8yGc1D333I+jjp6Ok086Hg11CTTWJ1FXnxDsNwlFJBkawSTLwc6dW9EYqqIhlUDLEV+Aoddh+9Z1WL1yPoaNHoV4cSz6t1aRzZdFlGe45E53cNMB8mU08pNgqjhEGv0pBAGJRIJvjE2GTvXkFN2ylG+aJoyUYCRFFoL65XKBG0AYurqN5o5ThuqTEI8HEY0m0ZfRMe3iqbjm2h/jsDFNOPfLJ6AhKSPATRVRZLJVbNu6DTv3tKOvP8tD4j7dvoenbM78ytlwAg727tmBq666ENt2tKOkUeuljVR9MyLJVoTCCVSrJkYfPpmhPbVxljWhWuKvCwUcaN+PbZs2Ycvm7dCp0lDVuT3PKyV58lIBB4dKTN6m9/gBru3aDh741TU490snoFrSWdsucnBxl4F8IS+kmO72qyV+vNzW4z4+rxxE+zYaoRo5NTU4mLt4DX7z6LvMNg8y7ABWvfwTjJh8HORwI0okc3Tfj3TbTGqR2o3aVGv6bcV+d8VGh7TmHSSo+JyWv1qozOvi1oJFxL33KjEBgzYKTwChhmQaOGawbEvcmYzIFgmJRArf/NJMtF94F2waRVozlsNWRH7JCh0XpQjqX4Wf5zKTzlnh16U3pp5Nd6KS2MjEDjJcF1MXPCUJRyx3tArDKVlCOBZGaVwbmm7/HrZf9ksc9tjN2Ez3EyIn4d48igdeGyaKxQJveu735fooMc90v9ddKJbL2L51G49E0S3SvgYgwxT3DQqqmDZlIk6ZNh5/fOJpzLrpSjQ3pDBs+inQ9Th2bN2MtauX4vwLv4Flz+xFrreEStXkcyAvLfS34jYbDPdpNCmL4l1JHzU4KIpotKZzClJUtZBKxQdrpXSlquREDZ2b3akcFKF7tsrkBN2eYZ6aaBAlgngyiFisDgMZE0dcPBnfvfpqKJKFyy69iG9mXd8Q5FG4VIMncQSlPnmN7ujXiAULluGEk0/Axg2foLuvG3FVxxdPGEN3H8KBjjzau/qRaBwPNZhAQ0MzO+ymEaPYwZKx0qhUijYEZTPpAaxe8xHynb3YuHkr3+FBqw6Vg7xI6+X0XsSla13bm0vPo3SBHvNeewwtjUGYBh2vN2mSFFNVvpuBUOQdXCUV9wcWZsOTNEXB7J8EGCStJGfgkYWPvfgPvPTOBkZF3iMOA0te+wnaJn0JUMIopbOD+mRvj5Y1ocOujbiC63DFF4ccn2e4h+qTa2G21wLLebB7D2H++qW7r+S2Pmb73JDJ0xFNaimjmh01lBNDClxwwYXofOQt1C38DDrlIq5HooM16Z633niaGsMllVmMJt7R0bu1XVG3GpoEIFg4TzNLKllvSBqJ/N082O2fpIhLA7H1VAL1L9+ODedcj8SFZ0O+9DR0D4hiOF0fJr54lAz1xgqxN9s0T3OUEY/IaGtOusSYmJ5Bf5PJVZDO5LFp41b059I4bGQb/vzim3j+nmvQ3JBE27STYZhx7NiyFeEAsGdNHunPLKRzFaJAxYA6Zkf/D2vvAaZpWV6Pn6/X6X1mK2xhC8tSpCpNECkaRIiKKGpECEaTGFvswW6MiUaNvUTUGA3EgoogVXqRXVjY3ndnd/p8vb+/65z7eWaHDf5y/f/X7/PyYnd25pvvfd/nee77Pvc5567Okfp1QoZpZ2uSNz4Bps8Uk3MkChcf9aukLcqczpcRJC0Qqa+yHdFET5eZk0s2x7GjAmPYTuFxVEY6E0Z7Wx+mcy2sfc0qvOb1b0YrKOOyV1yGJYsXorMtivZsm2h7nekU0tl2RJKdQDiLeqiGZtWECZzAMDP6LKKFHRrSzLGos9UwxvPtGtZGVgkdL3sXLlHGwJqYLUQvp8zlpnHfA/cht/sANu/cgUKDtEBGbYciO902Nyb/L2TZtQx9EOF7Mf1n+s1rvP+2byOTpjcV+eVHjMHp4czD4k9tXLYIvcPin9q4HOotzrTQ8xre8nf/iKf3GxjnX9dceDw+9u7LkV50EoJGHNVC0Y1PcYMD6EzqpkL8v9y4mmPsAUy3cXXYf++mNyriCjmjEXeViCbnzhjTh1pWCr4TkTje+JprsO3PbkK8bJpXOdITTSYSKmd892JYd9pY/lwqEhNYpAfFDyHp3xEfKv4b00Iflf2pK8DfnTSKlVqknMERRSQbw/BvPo/Hzn87mh0pLP3Jx/HQkxvQ1dNv6bDT5Jar3LhszPOhW7pNjPCpDU/h/ocfxdmnrsXKFcegr7sDwwP9yKSSqFFTWq1g4zNbUC7PYt3q1Qg18+jMJDCy9iw0Wl04sHcvGjPAhtv2oVys2jDtqi1e/g4PRrGu5QHCF+VgbOewbJBDZjyqw6RULmHB8JD8kxlRBfTxMGUJ0mxq8bLO7ci2SeqXTFEfax4NYn9HCMxwpEkL3b19mKrVsOrCU3D1tdci3hHBxZdcgHQ8joHBfoyMDGrIeCKRFuHC6249+OWf/9jOBxCrjavGIb2QQpJqPYotB1tohNpxzHHLNN6kt7dfzp78OZFMmk3kCtMoju/ELT/7DfaMTgrc1CesmyeTRSXvV2aHz/ya1QcSUmp17dEQ7vvVv2jTUoTBA8Be5jEldJ4JqaslSRDxLUBRIqVNdlxheWs9v6+aITDFz84MslHD+W+8CYVGCKEmJ/MZ+v/Aj96PJccMItK1As2CaaT5rlEHlHnRvI+4z4/99mntoLXfPT+d9z8zF63n/bA3kfNtOZJTcrOzCH3rI1dr45oEyfSbQv9cjUV9bDVo4lWvuAKJ+3eg8tXfolzhsOqWLFcIHinyOlsSF/BslksohAy9mWnpwtS4BbFlJMTWyA9nq8oeYcvpK90GF6+TrQJ/ErOdIB1wBIloEvG2BAZ+83ncdcENiNbqOOHBr+MXv74DI4sWO8M/A6c0woMR3cnnWAs+/dSTeHb7dmzYM4njj1uJbCqJamEaq5cMYO2Kxdg4VsepKwdQZe3UKGKyGGDl0gH0ZuNYuO5MlMpJjO+dwYENeezeMIoarVnrAaanJ+eQZInznVuFZ+yQaMD0K0GATTrcCBrNGrq6utTKKJeL6t+ypBDKzxS/0cTM9AxGFow4ZRFRaLPaoVuj2mkRWoXS2qaB3v4+NDmlYVEPPvrJT2Dk2AGcfuaLsHb1Wov4PDCj1NqagyafA58/a+tcLq9NRET/0NbfIlKn/WkYyWQW1GLICxsxHJyOonvxaeju61Imtn379rk+KNfR4Z2PoDM+gV0Hm/i3798ubWpUm9D0snq2nPLoDmXeE3HfSXF06LsypGhcAN2CgR784gc3CYPpbOtA1fX9mYTRUZIZCEOB5y2bx7IbSSLFljNadwHK00l9nCFH2Ud6thbOvOp9qJEp1YqK/94KSnjsJ+/HwjUnI5TsQok+TgoqvOfmeOqHVv/fNq5tWPutz0Odj/r70a0h/71+MAFLE23cud5SyBrkmprt5nmSh3rM4mNwxZVXYfMVNyFxMI9yhDR3jdIzxY53p3cnmZQ1gdmhhOsEYQIEZAxxwyLkRNQEpqxtxF6ZqXNss1oqaVHba0G5+Yg0c1GlYmkk2xPo/eVn8ftXvxvZyRyO/f4HsTcGlDkpQJC86TvpFkG1E69ndO927N+9C3fe9RDOOvN0TWmgFLGcJjlhDdKNaTQD0h3LSKbiKFcpK2vg0FQZq5f0oTsTxcDKU/DcxlkUt7eQH6/g8MEpcGod20iVWlHSMtb+vB7W5MpmXJSx4VQ0SuNwZx5CQAeBKKlDGGHJ260jJZaYWfLQRYGqIbUbdMDVEI4Ekglq0gLR5gR7rsyLqiDvOdTfiX2FGRSbdSxdvQixBEn8hkgbG8oOQLHaHNWO6b1F2zqmp6dQ3H8vx32pHKBgX44VkhE20azk0X7shagkB+R8snXrVr0v21FMmw/veACHJ2Zw2gWvwdo1qzA4vEBYSaRhJRmvSxFOuAPlfkckfWSzsa7l8+PUP94bfvZjFmVRJZ+8JQs/A/doMkh2XIuHc1VMOO7XeqWEajGvsqXZpJj9+fFPQWWeoES2SS7D2bx9N66/6WaUajzsSSwKY2Aggd999Xr0rXopmmHSHE24ImN4d//oejL/PV8o4v6/2Li8Z3KO/M7HrtHG1eZl6sshRw1LPfggOX/0pLUnYnVyBOUP3IwCpVPhEKpEbclJ5hnujjAPIvHWZhNJoau68X6AsenEjEUTtsl4Qu2YsGmh+ka5a09pELmrizgtLm5NegNzsuj+wXtx/zv+CalDU0i94XzEr3gJDu4dg1YbT0oynypFjO7biX079+LB+x/FqaefiGUjWVSaKUw1ouiMtHDuRWcgGy9jyzM7EImnFfXa0hFUa0ChWcIdm7vwjj8/C0G1iR2PHEZ9KoI8J9FXgWKpigpBiQCoFHJz4BRjgJElzMmCC1GqKkaXaEz96I62jO6B0HUnvZODR7lk8j2SUFJ0Z3JSSNrjCHmvIx0nfZAHBAkSvCf8piqGhxei54xj8ehdz6J/ZSfifWkkmeqKceVSSPc8dLAgsFm3bEXVyzg0MYG9G+9DWyyHRCyJRNJ46VznTOtJ8avUm+heeQFqsS75aG3e+Chy4/tQL09r0PSrX38jhkaOweiuWVSmSqiXWwgaYSTCSQcSATVmbeQ/Wx9HBxEPEpZcYs0xatJ1UzOrbAazZYYE/VxfWzArwTb+n7RrJ1GMRhBLcqRpCBEePHTWFFehhuLMKAq5GTRKBi6RgJXiemlGNIPqi9/5OW69Z7MkmUrqQ3Vc/bK1+Id3X4u2hSehUamgXLaNKwsn53c2f+OKduvCuaXE89qj7utHR1wf/Y+Oxv77+F+uHw6RV6bCGtejwwTD6bzATgM3pdDRRh03/PW7cfDyT6I8OmGm300OZnD6xjDlbNbw9myYGNs54pG63N6hajYo2kHjpInF4oqOCTGirKbWAcKmN6ODU13we+gvNIe+hUNoT7Uh8aXr8dQX/gPRzXvRXLcIa778Hjzw8BPIUGGEFg7v24Otz23CHb/9LS6+5CL0t8WRbx8GFq3D7c8extKggPddPIxYiDV2BZs27UGUJIZ0CskUS4YYRpaegFhyKWrUunYPIRxJINQyMrwUILocuyamv6qtXKtCaKZzYWRWIeaXAqlzkaCG2PppcyNLXTFk0yO4aOmNWaphfHQc+zbsxaFdh5CtAbVWHQnqiNlWUx+9iXC0jmUnnoCR01fhrp88hMWn9KOSILMqjUajMufQQNM1LgJ+1q7OTul9efJs27oZDzzwAFr5fThlzSJZtCayUSREkifzDPLLLlXr6Ft9EZqJbokAHrn/12gWD0jBc/3ffBj7dszi0MYZhMoxmbrFIgnEogm0Yuxx2qTCZp0m61XDNgIudIIwIsJqHXBTZ2iUJ+6xH89iYBEzKfWB4zHZBbFDwVKDmQxrYvbGs9k0SpWCEytwsmAOQbKEdGcYi45bjL5Fbdi+8THEawXEU3EBs8RrXnfjp7Fnqq55b7RbCocS+P7n3oALLngJQulhFKa54Q3V9mWcNyb0m2+OSDS3eY9syxfasEf3fefXv/77eRhQUTU+Pm4jbpkqe2dEblxGXDOlNqeGNWvWYH3bEoy/7WuohWtqEXF4JS+S6CKlefyzr5OZdoQbHIdxhMblp5dJRO6dLlwkFuLqmE1e6eE3rgqoUEh1sU/ptEVcxE1+8W3Y+NVbENm4E6GuLJbfchMeeuAJNMINHNy1HXfcdjtefNrJGBjuFEmkmBzCg6FVSCfDKI4fxKcv6EQiYY6J9InavWtSiHMknsWy1evQO7QS5UID44encHj3DMKtjJz0GXmYlgXse7vDlAswVDEBPr/Eg4douVwe7Bh1BAu2TCylo6GYvJeUOpo3NR9QNmNDuwXShKugq3UoHsbgwi4MrBxGOEjh6Z88hqlDo5oyoEjVaiLbHsPQCauAgSy23XMAx5zRi1y4hFYoiliUtaWz0E1nlG7RhJ7kiWwmo7bUX739HTjp1HUY7O3HxN6NOO+01UhlNULc/KF4knLj1uoYWncpCi2qfkJ45rHbUchN4Lrr34MdOw7gwKMB6rPMMmKIJzkegrUr3TzswOJC5zrh1AFNwZCYgCouIpos11rIZGn9a4wrDz4RByFZhPeUG5seZELwJcYgDbQmmihpsfVa1cayhO2ASkVjKNXKRvmkk2PvBE695HTM5HehNXtIffFys4lXXPtJ5Ko0g6dpQ0ssugf/691YfNwZCCIdyE9OIuxYXv9/Nu4LtYDmDvIXiMZz9S1bqAHU3hRH++sfulpjNj2STPiZtSajZritDW99/Zvx4OUfRv9YFWUO9Q0a0qgSU+OLaTLBKaKfYrQwySYfmYvQiQV4E3giakKd5CG2uAVUaSaa+RboQzohtUcWiTSL7ujkfiZcCCGRzKDna+/C/f/0HXRs2o9qGFj/u8/j0c3P4cdf/yZGFgxh7TFDWhCToTZsjS/BWGoY/ZkqTurKoK01g/VdeRndNcNRKW9K5SaaQRYrjj8NhXyAJ+7eiWY5jmSQRTJK07KyIoD/TLwU7+Mk0MWl+joI2f4IkRTRpl6sH0rFQ0pqGA0Kt4jryfY8LAlUkQ7Jr6kH7HqWjteGYpBDrDOMky9ah5n903jqJ3cp6nJywPpzTkPn8Utx/2+eQKsUQd/6djRTVHwRjmiJWcWDktzzvr5+/W4DxUr45Kc+IVLGmtXHY8XKFRgcHMTeHRtw0vJ2tCeJS8RkYkcTOtIQB9ZehUaUHtoFbHnyTrz4nAvR33ssHrh1G0JFNwhOPttpM4j39rFaNJR5RrV5D48ddqbvtBsS4VkHisz+3ARGmRQ4RhXvC1NUlnEkPtAhRL5ijYZkebzn5KdzQ+vQ9JMfKQ/NsvVWNgAwEUE9lsOLXnk8xkafQZ3jQWeKeNkNXxDhwzyom+iORXDHTz6AoZXniAtQIoAXCsReYp7N0sZrjL0HwP9oBx0ln1fsOYqk8UKRmBuVpRS/l8+N4KE32At9+X1XBfkCJVGqpFwqA4TjCbz+DdeidNcmFD/yY9RpoK1ZKnVUgiZqPI3omsHZn0ELiSgjp9ViVGjw3eYG/BJVZBokiVgY9UoVWfZ2XfQNmnWxlXSvnG8sN65O5mTK+nxOZmZ1CaV0WQz998dx719+Coldh+Vn9MiKOFrr+rBquButekH1y2TbSvyu0oMgkkF/OoorhktItKYxsmBYn5uACXW5zAZqzXYsWXkidm+ZwdaHJxEPEmKRifwgIoQNreZnNA0zU/2q3TkN3wqLqcVoy4g8ODik+lcnqrdYEXKcVirsWVSMsvTnGh4Z0kMi+urJCfwvFzEXinjg4SjqdeZGBay+cJmMCh7+7s/R1tWGkbPWItXXiQ2/26nIMnBSL0LtDVTqVZvQ4JhoKSmh2sxxolHRDCRGP1r5DAwMoVgsoVQsI9PZhf+6+WZc97oXY+FQCrGALpxllGsVLDj5GlSDMPYeOIzKxG688rLX4g8/34RosQtTM9OWlgvDOJJteDCK94MHGw8SbsDZHDnhZpFLbTP71myRzecyc+MKvHSjZmy9UOJY0+8hMkx3UOv/0kPM7GR9RFd0VvvGPLzYimPWkRho4awrTsOOZ36DbdsP4C8+/E2Hu9iOeN2lJ+Gjf/s6tC04AdViGZViSZx2yhI1b5FtR41OsbzghV5HGI82GfKFXkdvXMtgW4hHzR2T94Ke457aGvrSe66aG2wtIUsQYMGCBbjqytdg9y8fQuXzv0S4WBYPuchZIZzFE4ZQ5fkblxvS17UaHiKKoYnHaRKn9JLIKf1wqf+UCNqRwnVCBjYJ0NW53KyefM8Tle+p3J4pJ10gkiks/cO/4t4L34n2XFluE5lLlmPy5Da1UHhIFDIj2BJbiH2zUVRTKRzfHsKFg6PoiqYRontEKY96JIUo+UHNLBYvPwObN41j15MVxOnWWGPmEHIjNG3TKhJyKnqCdVtMOmSypJQ5hAJtVG7c4cEhM+d2TB2zPJUd4ZEeYxh6H24a1mVqkRklfq7eTyWSSmN57eZ6yHlABiiVG2WcdsUa/OG2u7F8aAiDJ6/AH371OIJiQkDMglM70cxQUxdIqmhtmADt2YxcHSbGJyQG2Llzp4gqmQytUt2w8loZPZ09+Mb3foBzzjoFs4f34KLzT0BAMghaGFl/NSrNAFt378FLT1+P3c/mMfF0AzFwYqD5dHNyIfvFVrMypbeFLvFFyAzQLdMiQ6wsVRb/3ffxGXG9nlrtaqeMkiFBzAQRsrVNJPRMiMlYKspWkrH1zB0zhnQ6g1yBEcs5PLoh6mwFHvfKxQjFpvDFL34B37rl0SMbNwC+/Ilr8KqLz0couxBT4xPKquZvXIFSDmT9U4L5uUkTDoQ8OuIeDUhpDbjsjbiJ16ITmCI+0NPTjdC//M3lQaVUAZdYR7oNl1x5Ffomm9j0jzcjtYXeUzU0WpYYS/3QMgd+3nKf/un0m0fnkku9NquG3ZieViMOzU+XD0fTRwlaOSKab0kxCul7mSI47ylRvTiPxonr+Tniqxah55sfwtbz3yn0mLDFeHcdnTecIiBmJ3pxqG05ikELhXoCK3szuGgxhxGTwUPheVS+WqEwD400+oaOl3vjY78aBWdV2pxdI6aoZcUSwpl4+2xCEYQaWDXjAY4rpTXr8PCw0nn6RstbqkHXCjOCZy+OAArbLpwLxDRWEr6uDkUfLbzA1CqKtGSJ1ex3mzyR2s8kIrR3pd9UuIizrj4VpYkxbNk0huJuShmt5ZJclkMrxjQ9QDbZgUjcrGjp7HF4bEKLvrszi/EDBzBLhU+oimxbO9raOtRZYLP/jxuewvihcaxYuRLReB0pjcoMsO6Cq9UJHCBIAAAgAElEQVQymZmewmknnIG7/v0pRBspgZoh9toTcYyPT6hdxA3EqMQD1RBiUwlxbXlQjwuSm4ByT4/K8qDXuhC4GTWXlgZlf+zvGwmDmYW8tJwzpt+4mk6hEbCGkZgtEbM4Z41LJls8pjWFTAtnXrMeZ7zkbOybkHjYDuJoDPd8751YftK5CIXimJmeNhFNxAziuUZZNhjZwzJB/3p+BHXdE/fPR9JkI58cDU7Nj8g+TZZE1Q20Y5kT+sxfXhqEolG8/GUXY0FXP7Z88gfIPnEAiLG9URJqR40tdYdawMT/ND7DFrTAJdUtR6RTcdbIRN48b5OFPp35aMjmUmEvPPDjNv2HZZ3X2dY+N3PFEnjrmc3d0FAU3R98ExpL+rHv+s8beMOJ6h1RhG5chkIrid80jkU51g+EGzilK44Ll9MKLySHBdY4HBAtCh5bK23HoqtrBX73H88g3ezQw+Tm8iNQdPKLJGCgiGbUOuN3Xg8JKeoNIkBfX49NDXRRmJvWxlJwIcXQ5JAzDTQzJ0GK5tnL9SMuuPDoDOIXhr/H7A8zmvO9bJxLSDY4QTSBkRd1ITWcxnP/vQNNKoYcQr/otFGEMtMAUmiGqkhEF+PAnho279yp6fW7dm1Dd3saixYtlJa6LUtKJQ/hMA6PHsbuXU+jWi5icjKHgYEBtHdmZLNZyE/jFdf8lVojy1Yci8d+uxWV3TGZqzPzSZEt1uLIy5yMGFiTGnvNi9RscBkPJj5XZmDcyOxZlwp5JNlXdb1e3Sj18zm3iOJ7+mZXnUtkTPU5D1jzFPRjVRtKhXmfaErnN69lR3Xpodkvnxu3GY7hhCuX4ovf+Ta+9u3vuh5zC7FGHU/c/gn0H3uuDO/JWOIr7twcuaY5YcOCjnWXj46e8xFiW7+OeDLPLfOFIq7/mth2kTDGxsYlmeTfOzs7ENp730+DdCaLrR/7LhKPbEfAcQrxGKLsJ7YaKIUDzX5Viurm0BKv4wf2PFOdmvOkSxoxxGkFvi/bbBmpgIQNN6uGIBYXszyC3Ga2E9R0uCKHa2atG6I9r5iPdLZj0Z1fxYOX/TXaxnKgElgT5RIxzFzei4cGT8CziVWoVetEvpCuTuLCkRZOXpxGF3unjiLHeB8JJ9C7aD0ev2MclYNEP81VkadxscjhXdY3thnABKNs4zI6yhSedjq0gG21xCUmMOLBJ14Pa15mJNzAFBkImJE1KRddWUZvZFzRelSCeicwn9u4jv5otkIhtLe1G72QJu41m3JYQA4X3XgB7v7GH/QZJUrnwh86jJ7hHrR1pBTBSRlsNCM4PHEQd999L/bu3YXwzKSM87bt34cgTAM3G6FB293ObAsz41MYXrhIRu2DA0Pyj56amsAp57wSmWQCQ0OL8Pt/30YTSW2uNGcAhSKqH3mdowcP6cASycH1bU27S+F7RAcRa1NGHn7G/OyMwCZ1J3g/2G5sNJFMWDuwWiObyyYYWDZk9Fu2lqjx1s+xBEnSe8zsivje9LYiqNTb06PNG43xWVuGw2fYd0oGQ6tH8PEPvFeHAUe9DA924UMffiO6+46XXJMHC78/6e6RDPfnlE1cVV4PfIR+8T9BJ2c4f9Sk+T/VJlJLMBwSHsHrZ7Yl7fDjb7ouaN2xUYN6a7WyNgwL+UqNIzUomaE3Ygi1SADKhllnJTvbEe7IIDLQhXR/N2Ld7Yj3dAmsaRJYODyB2uPbMPHYs8iQjsaUpUrChiBl45UKKWa/17ntuIgtNJoqHl27m+cTCSPWDKEWbtIJHCt+9yXsuv1BlP/lZ3pPotriWUeB8RdncNeZr8e2mTriLT6YCBqoacpBfnIUo1u2Ij27F6evW45Tl/Tj5DPPxvFLT8bjvxxVRKsVCTqZCwgXlmeqJOOM0uZIyDRQIzUpgo+GFTm4YJgGcwFp0gPvm4EGQq40zZ10zqgza+fw62RMvTljLFUE1nChOeWfO73JeGqoDibSq1Nehx9TXqbzYYQTCSw/rxfP/nE/GhOMygROmug8Lo+Jwqz6uByhOjDYi7vuvN/8nQHs3rMb9cIE+jvasW+sgqo2SgTFUlmeWSesGsHCRUMY6O038If65MIspmfyOO+yq7BwZBjbHx7FxA4rb1hrClGvtnRNqs3CIYwdHtN/6YU8xyHmMvfuIPPMAhltZ2dmnJrK0Gmqd/yMIf6X78FDQUZ8bnCZzdYN0CZdrY0B5YHBTUy9LjcpTfdsdpUNPVOZ4xVunU2cfc2peO97341GuagM6MY3nouVJ52JSKIbs9Mzc4eFNz7nNTbny/H0TNxIl3kg1PxRKKZ0cbFX5aOjP7qRKEfSZJskwetkn533ngc761tluRte8cYgTOJ2bxtiw4PILh5Ez4oliA/0IKDUjNGJ2A0RPBb21SKSDoXNlUuIFmuoT+UskhIFI2gz0I9IbwfC6QRq20ex7X3/itkNWxBiZCKn2QZEauNycr3YRWwhEYBxHj6+leRPoiDKTR7F4q++D5W+Lmy5+iNIShroke0AzWgNtXOX4K6zLkYykcGuXXsw1TmM3Ng4cvkKipNjQKWIanEGqWgYX3n3m3D6iSuw4fdTKB+MolTNIxqwjmqIoSKLnURC/UHR3yJEdFl32onPGoosJ95QooyVkknQBMTQSJ2UT5dS8+ustZjCsfZltO2l/pe0OWY3NTeaIx6VD5ZSMpdicuFx4xAp9TU3nRrIGKpV+VwiCHdWccqlL8J9P7wPcW3cFtqX7kI9xujSoUl3iXgffvGL2xGJBqIVHjp8CDu3P4flxx6LHXsnEGVUk79xSZ/vjJOX46KXX6CevDjfrQAHDh7G/Q8+gnf+7XuwbtUJuO+H29CohUWW4EHH961XWcuaZJGZBaOd3RPLKNQCc7OMtZHmAZK8l8YQmhE6LL02HSBr1TmXCsM/vJuGcQj4d66neCImuirza1Mr2ZA1yva4eZUdaoKCpaCMvk0iJJEAZ71hPV77xrfg6ac3IBEK8Kuffhgr1p1HiY2ki8pEvP0OiSBcz/Ook36UibKBeYPc/yTpQmCVi8BCadyGdoeBzZ6mCQM9o61t2Nvbq4MsVNz8aBAlW6reQLFZRf3gJMoHJ1A8cACNfeOo7h8HihW01YFEyShq/H5uVHoReeYo0UQ9DGkDNSQIhZ4U+j53PZLrj0PjqX3Ycd0/IL9/FNVIC9GggYBEDbGJGGEtFQ3XW9b/dRpcAiSKvuEIlvzb+1BdMoznXvV+pAnkiDUUYUmmGTitSAuVpXFEb3gdJlKduPWJLVgzMoRFmRB+eu8T6FlwHPYf3I/JqSl85f3XYXEb0DuwDA/8ZBtaxThK9QpSkagE9IV83vTBjiEjLnHDVCxWo9oCZI3KTaVIosmAPO2jQpsZidOufuMjYQuG7QsuaAJYQdMDGxYhuGjzhZy0uXygXtbGRc/+rlEnnS9XiykkQas4CuUmcuVJXPjOF+O+7z6MRDylmvxg7RFUgxksXdSD3p42pNo68atfPif8gqNhxsZpdhbg8cefRM/QYkVlCk34+fp7evHRv79RSp9GPauv0VvqmWeekoHex2/6JA7tmsahh+toxlqyzJEEjwPf8pZ1SCpaNwEBN7TfuGrvhUyJxsORm5cAH1+WxlKvTTKLlWjcvKQt8n5KJSN02uSZYvjxz37gnEa5BhpPyvfnUG/+Pg2Uc9MgmQQJT9U8ZANRYqE4ll3Sj/FaEa969RXoSSVxy83vw9IV58mMPed0wb6zwc86f+Nqs7oZODqc5m1cX+ce3bv1I9TtGv9nes2Ny2ucnc3NXXdfX5+yr9Dm5ecHbOVIhkeYnWJ02qW6KQJmim3oHm+yRyy9IZbvzVH87j+gDUI2rx660U8tG8Sx3/kAKody2Pu6j2Ls8G5EeMCQVyYbbsrd/HR2MmysnURieoI1SiSMVT/6LGYSUWy55mNIVmpiO/Fw0Oeg6RiF+OEmKovacOjCfpSDFEIa38ETNYJnn9uCVjSFBWtOxFvf8lY0y3l09XZgz7NFTGwMoU5fI9rHuBSYD51/N9UH38FNfRd7xxYlI65GPc61tawtxAdBAMWnYhQFsC4hH5cnd09Pj5kJcNE5/2iJpVyflWZxdnABhWJOp6zIGCQhubqfMct8p4FimdMRSzjzTevw8F0bER5voRkJMHBSGxBnCkneNr2CiyiVCxJS8M/ymZ6ZwMMPP4zp6SJyRdqj1rFm1XJce81VQCihNLNcsYHRBw4ewMaNTyKIxPHtr38Td/5gE2qzTWTiaYGXMqCnVRCZd26MCwlRfmqdoq7v73O4tu9E8P46je6R7kJ07h4yc+Gztt6mn8hgBxjRaCmaOKZlbjoElWZxgX6Msha5jcQhQoZYpm5Gs+u/xmMhtC1I4ZTXn4Qbr74SSxd248Z3vBEdXcv1zMj8EnCo6Y4WGXmQNI8yjffPf370nNsXR1navFAk9lHdZ1xcg7OzU4jH0+jKtiOZjeOhDbsR2jF8WsDFwyI7iETF9+RN0DR417f0fsg+AglPcnUSf5YEhQa9drxDvktd+MsF3bdCKHTEseTXn0e9Auy+9K8xeviAicrZD9aUPWvUk3qmjciNQWL1QD/W/eJzmNl6CLuv/wLitYrSdvPCptmtsd/VjkED09kQUu86G/UgpgiIUAxVEtejcRy/9hSk27tQD0Kq45YvW4E7b96K+rTV2easT1vXqk1m10gQWr2S8eVsNx1pnAuIG6pSKllaywdaqwosUvrbNO9gno6U4VGXq9qLM3Gdo6GiJ9tjIrAcsUTlkEaf1hnQktT9MGGPmyCvU9oECoVKE7VyE8klUQwtH8LuB3cp/Rs+sQu1cFnti6Y40lZ/hee57BNTqFTLeOLxpzA6ehjFagV/dtnL0dffi3yRQ9PIC45q3vETTzyBZ595Gu/54AfQmx7G5jundEBX8iWNDNXcqGQK+ZzNOubhVGYpxSgqK16boKgxqxK0WNRUNtM0b2hLr4lC26FuYF3UKLbOHI4/M3dYzpPqcREoisfCstvl2iJmIMojPcyc95g8qmWfaxE3FqO6KowgHcZLr3sR/ur6t+Kay0/C6eddgFC8R1MayKbSQeHUVUqx2XP+Xzau750fqV2PpMPzI7A/sOan4irTaPlTt4O8Fs3gKz/bhOem2xDaNHgqoTlBRIlsB0qFgknOPKWRBueudmWNZrpdLmZyROviuYrVMs9Amy0Spot68eTl/ygY7+/C8t98AWP3/hG7bviUhOPynvDDmIhcq94Io0p0dvkCnHvLv2L/rQ+h+PF/l5skHwQfojG0WmjwwYQ5cc82SzEWIPb3F6LElhRqKAchdLZ1Y/W6U6SxTCTbtFAr1Tz6+hbh3u8fkvsEGUnarLG4alAeUlxk0sSSxVUlFdQWAaMDCRMiELgDTO0Od9AZsmuTzRmpIhGjdJL4bv5E5NUSfY45uR0JCXa7VHuFjcBgabeBLKI8ztu4/s/8mVKtiaCWwN7pvXjVuy7DAzffJx/g933hvWhGK1h3/Hq85JyX4OSTT9Z8XSL3/sXowc1pw78bGlxGOI9Dy1PpNswWZlDO0ySgomvJFwt43TWvxUO37kYwDkSSEURaURwYPYS2bFYHmEdguVa4cf3MIhkpcGJfqaxaX1lZk1pic7rgywM//C8jJn+n7oNvB2p2kaXUtnkt+2HGxAjY0c5h6GYazx6hGG0uvfZsNNswFvG1sUI1RIMkamHgnL9Yjb+4/m34zHsvxaKVZ6IepDA9NeUAR9u4foC6aLn/y8Y9OgL7++5/99Eb2m9cHlgqMXj9AL720434Y24QEwViDTWENnSvD7hYSMNTTUKrlFodcaF2lk54l3XeALoh8KbJPqMVCBVVGu34lJ5v6rWJfuSmasBICIX1S7Hi5n/Aczd+Hodu+TXyTdZIDeRCdfSduRb1YwZQ6+7A488+g4995gvY/a1fIvjOb1AVS8Z8/MyTwOSE9Le1ifI6JTR4KvyBl6EQM08rpn46rYMYCvkiDk1MIZuK4uVXvgm18Qx2PEI9px1EPIHN59ec9326It6sSBhmcs62j48MjOp+M9shZK6MjIRcpNygpBiydh0c7AOtVkj+kEWN7HCNtxximeKmETACcWAZWxeK6AS6KN+LeajyiIsgf54G5PVGAuNTo7jk7efgnlseIrUNn/n+J1Co0eOZEc0irmcrEcEmJ3jJ0iVYuHARli9bhsULF6BaLQlA7O/tRyrbrnp/cuIQanXWcFAv94Tlp+Cem59BiCNA3QAvZmjjY5OqBz2SzoyIf9dBzpTWfXylxUqpbRN6Cx4PXGktsiSRQZo1ctm+4cNXhBb32owN+bM8ZEkHnNMtN41ooXZT3AlmJK90UdNlhp5Qw94+sZZWDDj9qlX47V0/x0vWZDCw7Cz16GlGJyKEk/ERSfb8ZIa8uZcfseMMAvzX5+t0j96oL7Rx+TZJSr8QxbPbD+PLv9qHg6UU8jVzRVHb8I+dJwRMdRX2nfu+indnpanUSu/uepmIIJPNGlDA044pjecoz/NAtjEgNj6YPTW9PxUiyRjav3gjMievw8NnvgWPlHZiwaWnIL16BPlwHcVcXS4Df/6612Pff9yN2uf+U35INqjKUqRQJCTnQHF3xY6x/IDyLk4wr73ueNSWdYKGKV6Zw0lqXALcSATCzv+za3H3Tw8gyMclVayWbVwJf4f5TBs1T3B8rarygWkw02PtAvV0G+q/8iESoCIyLKoneboBLWksarK9RNUKwaVyqaJoEwoZ19lHEppwC+yS2VxNhAfxo5kFxNkHroi6d2Riu/GfmU6VK1Xkck1Um02cdtVabNu0HcXDOdz6wI+Rr+VQKZeM3FAqKWJUa7w2ShkbqDWcOL7JSGtYBqmHf3nD27Dm+HW4+977VAotPfYY/e41x6/GjgcmUdlPIs6RXj5XSblECx8TSIgHnEza3x1ZXlMYnTCeRAulwSIYmK2PbWKTryl1pl0OBRoaMm1kH2mUE2wT2SHEDIxAIidDSPDh3Vy43pzxAIejKdWUHJCoNYOSbXrNIpYIhusqitXnD6N9aQaNyWfQ1rcMM7PUWFuGoo2rWUMmO7RQcaTv4109ZBTgkGGTeBpngRf4pxDmuU3OSEvmYTyKJ3fN4gu37sXBSgwtMtmcvluQ8PaFZwWMND6q+NrBi9z5ht7T2Gh3JiDgQiUB2tP0vCujTjFnJcn3ogiBvFoxkfhQIiGMpcM47tF/x6Z//B5a/U3kO6pItqLIizAODCxchf7+lRg97+0oRo1iGW858MrdFCmSeFNIkVTeaF5SzWYY+XOHUDttRHVdXIO9OHzZmvH8fyiUwDkXvwl33rwPKQTIF4l90EW/rtYF6zRuRn9PRHiI2Exg1V8y8HKDoV3tleXh1zCvLhFTGk2UikWBeb29PYoYrOt40wnvc96Q0mKJ1MMInCkY0de2bHqu9mUNyujMdJuR0JcgfjI8a+RymbOKmogk4lh85iDqrQp2PrkFO2Y2YqY8Nec6yefC66rUawJcKGzIFUwEoXSTwFzdOgepWBRtnV3YuWePWKvMXLhhHnv8Gdx/8xNIVJJoeHsescZ4qIZxaPSwFrgGeCkVNbYcRRfqx8aYFpcRi9hnkRjdWeYSwPOkHgM2LYVmfcznpvqVLUNHVmHtx03d092tDMhHRf4uvg8R7UJxRlGaNa7MDqoVYRlkonET8XdywwUtHrpJBL0VvPQNZ6M8sQHRZI8GmvGpqU3lNq7cT53BocwU3ctvXPVyj+xEy1r9YID5fV+vTXcBT+HRIcy/uHsnbn4iQEnG+mSlMYjYgAAZL2wbeXHg3eOPuOVTQGH8WHvNS0c1IdMkYr4RLsBhvumzZqtyFoy1dhjFuAnsQ4WM/H3Tteh62ZnYeONNKFzcp5lFjN5M+84470o89fpPILNv3JRGfGj6PHZqeU2vlTimnOAG4FZmWlw8phOhN58oK1JuFt5QZhNEYnlyvejsl6JcGMT2PxTN/5h80ybrIjvVuFisbLAHZEJzoKOjXRuP9SgXjBBOhwXIM+lIJiu6H/9dM1c5ST6bUdpGDrT3VmK0tihqtbOJEoBEzJm/sw/sFwWBnWZFogePQPvnUy5xQTY1d7htcRrDJw/juTufRiW7Xy6PRO+pKOLi5rUVCXhUqjqomLlYthVgZnpWYBrTwzotgFjr03OMNXCliVe97rV4yxvejg237tF9YMuDP2eZSRy52YIimqmOSDYxm12+uEnpq81SRBvQtXh4nxhd5C3teq8G2BkPXNarLlJZL5jP1MQwjMw017Nsy4wX5jJAx0BjqcFnxfKEG5iqI6HDySPOjmxTMbKr5xxUcfHfnI1qbidCkTjGxsYUxeNzRg4hOVZKoupagnMbd95UvheqYedHWz9EfW7Xa5hACPFwGN+77Snc9kwUJXCOFdc3cRG2FNxUBQavrSNn6dbyhPSsD90cpgNucpolzs4lj7rGpM1Z8SkB0zVK9bzJHL/XR27eXJmTs8XkjOi44Gb6M1h255fx5Gs+htClAyjEq6iXa4hnO7B2/YXYd8nfafFYP4yxVMN7TT/nUi6lzrx9Gi1CtQijRhOz/XGk30V+KQ8Ja5moppRWs4WXvuqNePiX46iNRWWA3ar7mTVO9+lGPnpvZAm7nY2qiFBCZ+0UjbvBZb5u44LgK5+flSKFBwY/G+1R6FAoET1PcEZS0hmDBhJxo8vxACToVasWHUHAeGWemM90sVIqggB0nGCca6fUG4xGtpFqyQrOuvoMPPZfD6PRvR+hSF2icrW2NPLTDiOPX9Dojv9GJL3WYFupLHF9IV9GKpm2A7FZx8x0Hh/9zKex94kyigfokUUFFrMB6/tycRFDkClIKIR8IW/SPi1u1pwcVGZaaoJ/Att0CDclJ/REFAMIY2JK8XkzQs6NJ5GayGYpMVK3yd6HaqmW2H5ztq1UshWZ4em3S3lktrgGRumQndNEM7BwwqOVNASeTvzzY5HoqKGSm7H+c5j4gqXJfLFuFxg5X1MrEc6RfXIk4DqXEx8C5xE25iv8WFLSNfPff70Bv34mjCJsrcTTZNORLWYZpR8eF9rYc3LA09AMoW0atxA3OeVruzqswT4A00XaWTINlOxOobuFbJL2KO6CONfU1QDeBI4nlOxbHMLXjAJDt34K9VAE93zpn5Bbau917LK16GyNYPz6T6AZNXI6HfbpRuBPLA9iPH/jUulBW506RqNVjHz6KiGkRCzllhCn1I0E+G6ccM6rcdf3n0a4FEFZg7isxmIbQ3QyotsyzQtEVGA08MwZ/hvfkwudJzSjH69JIojACAdMq9mOYOQiP1nc23QCcQIsLomSGUA0JtCKKCgpkh2dBnoFjaqzuXFSSXGlWQ5w1CZnzNuEO3+qRyIJ1BsRFMoVVCJlnH/92bjn+3cjMjCGZst41Hx/z77hVEU9Zc5oKpbVj6a/FFF7L7tT31JZQFP0R0ocb3j33+H+bz+HUDMhk3v2Ejgnie/L665UicQbWMfsoVwqI+nQdT4rblzrf8esNUPVUlsG5ZpxwnkPueG5oNva2sWA8tRTH42pIGrvaDO+tiR7jpghpxRuSOvTckPzuUh258zluL6Zdstt05Vclm14bjTvdxQDZ2Sx7JQFGN21RQe06vK4Hch8sa999MbVWpy3Keei8FEDwPxmt5T3iKVxKBTDfRt24yt3TKPcjCOIJBFTOUXTQmarRGts6IAyjyc7Tgj4ZppNE2f9YD001miG+pl3lOeYdrV3GE3Mp8H+w1Ijqj4oVTd2sZ4RI6GAH1btEDf++8xZK7HiK3+Pu6+4EUuvO0tCx2imE7nxMCbe83lw5LIALtYMtGadP/xXd8YAGlvUNiqF59JMpIWRz74GuSb1oLSBsUHJBHrWvvjlKE6lsfn3OQdImSRLvGOe2hHblKQ5cm4Q74e1dBghOZg6JldFLgJ+tpT4sG6siJvVyo3O+iuRsJaHShlXm8TiVtsxE/HaXKavRHipWJLXstg/bqj2PMCPN7ZWLStdZtS39w6bfVCLA5lt0PXZf/ki/P4/7kHQNqrIrFlznE3sRlkq13QvZlpGBpkHqBCwcUbiPGBKhSLOvOQyFEaTGHsir5q3QsM0URxJj6yq1ODGK+TN5ZKbiuQNuqIoGsq5xMAskUkCAmt2MDPSsW8tRZUiY0htHbqtGLBjBgV8ETnmNbJONiMCo5YqC3LtNJ/t6WASVdM2LJ+HodUWea1OBcLRiLILcYJCYWSHozjpVauxZ9vGudrUYwsqoZy5ok3Pc/fS9+vm7qwLe0fVtM9Ll2WPQ8JTA+OFMt7/9WcwjTY0YmnZvsaTaStnahzknVLGJC44p2Q81XWiM0Q3obv6Zx0dRn9zhm1EgxkxbWK32/FuQfkPwtOUp6IMy3kCayMwzXKsK9/2IJWP/rlM26IxDD/0Zez53I8w/qP/Rq1Vw8hrX4bCypWY/dBXbFzHESbY8yKubrxQYEvNvCkbb2YhEmDBh16J8SS9mDlBwMjvTCXPufw63HXzZgTTxkGm7pSfm6AUr52pNFMjfj91yjwRGAUZOVWXiLFF83i2j5pIa7KCcZe5CZi+8cAiwkzrVxMb2CEoml7UDjQtGNIDqUHVbCACfexvhpFgy0N1HdNJ+zPbavx3Rnv2q9lOESOI1y7taBLleoB6pYYX33g6fvuT2xFvnxQophaPi/TKkhzZRC09j37O+R3bBvYHN593pqcPp5/zMjz2090ojfMwS2rDMjctFug6QbUUyRpGCzWBe0g4yMThMRC447rm16391ZKUL58v6B5ZKm12M6xV+Tv5M1QCMRvgvWPKOtA/oFRZ6bHsd6lAMvDR9RVMyOEGirFNVMznRBflIVcu0zzO+uG85zyQxZVWORZGPEWqaAiteBHnv/VM7N35lK7DJKVO/0uket7oy/llpGM8Wp463+rC39v/8XWKM0KoBjV86N/uw9ZiP0LRhCyBSBhiek5ar9cQM4Mayi8AACAASURBVHD4/n7o8bbj3dawMYEecu8d6AOn2NFipCWWiKUTNr3MwJP5LA/Pu+SHZiriN7hpR63Z7Qd8MdqwtmLU7vmPD6KeTmP3pe9CuVZE6sozkDjxJBz84JcYQp8XZeenygIH3M2xtMXqRG6uYqiF2DUnAauHEYmF0ag1JIfqX3wshpedgSd+fACVotVdOmxicbUU+F9+RhqU8XSjAIK1kjX8WYvGEecM4ahNQVdLQYivqYh4f7gQWA8z/ybwwtm1mjQrX2PycMNSCvH3UnjPeyiuc5P6XLaEmggHpmG1iGoRhx+CRAmZYmtUhqWkXLg8kCKRpAzDOe7mhNevxR2/vAPDi8M4dOggkhzWrXLAMhih2O6/RsQ3FFbAm1hJtBgy2ilbOC+5/Br88ZcbkKkM4sCBQ2g1w2hv78DefYY4c/FyNhDbJpp84eieau3EEyLaGE/btMncJnK6cACWrF8jvNcFpBJsz9nmdbOrVfszI1HpIVDpyNgSUj0ZIFLCFpyxvxu0RrklLXA9+433T6YG6qNz/ZgjBwk/as0RJ6HzZrSC8647DQf2PWMjXnTY2cYV8eN5UfVIXfv/eePyXYMWfnH/JvzwwQaq4QSiqR5UmUlyJAoZhRHXVmU22QwELioDfaxjrVJlnbIOWPC6UD5cwuWkM1LELP4ua0K3YTwyxp8X7d59nYIFRh72Dr1PkC1A9z38PhEammicuwpL/u0juP/E1yA8PYP0Jacifcm52P6OTyFBL2JWdPOr+KNSETvdDF22YhySHx5a2YYlbz5P/s+ZNDWsJZxz+TV4/M5DKOyIiNHj60RNkBdgI4K247Ia+ql6goAK5XrqmyaRlIuE/TsF1lwwMioLM12kqZqRBIRiFktO0sfNwe9rU8bBk7PWrGGQ/Vqi8qRxOiYQf5cxpgi6HfldHVk7OOXCILsX6wmrhaLISxQ6jBUvX4oHHn8M0ehhbRIt+LR5J/u02DOUGHXmUNu6SRB5bcl4Gs2ghjMuvgxTO8vIbyG63kJxhuBVXiwpjprMF8qoVQmaMOMwcYGuwx0MJP9zo9EZhP1gblBD43nomEujPzQUTWS1aoZwJflzWUTm/3VfWTK5mUMei2C05+EkVRVxAL2HqYy4BvnyrC2NQdGAbluLyniSJlAnZkGhCbW/p752Ncan96NSG0cmQ8TbXprV67IXre0/6Xrxv6fKvE/8/X/9z/dgMjKCZrwDkWQbYikzDPC8eR0YPBQ5z6vsNOKPd/iIy2fmhNw6fY1Lyovv6+5BoViw2oSppXcnEDrqDMtdW0ZjMmUGzlMsKtXR3CnvLt4saQI0edGpOIbv/Fds+dx3Ubz5NjRWLkD7e6/F1jd/CMkghBjra3kWz+uXebraUTWv5ztXwsD+jhqOed8VCBJhJIMoIp1dOPn0V+DJ2yaRHy2iWm0iN5szBNNZXwpwopF7vaE2BFsE8xk87GfrnrA/rAFeBHNo5Ba3dNctBuMTOyvSRl1ZC9s+BFvk1FGyOpAiek5akPqFcj5FWRN80J2SiziRosVOzSRt/JqrRTV9SYveAT5kXcFqxkUvGcFMq4idW+7X93PR0ZXCz/eZnx7z+0WcbzblgMHPxgxgejaHk847D6F6Gvv/MIFIPSHTuVYthG3bdittbYU4gnQXopGEEHxrCxGoi9mfmeaqN0y9ctLRLW0DMt0XAUL6VcMMZLimdLklVNk2vVFRBeD5WtlpWg1INEsfIueWNFgLju8ld01xvK1lqM3A9l7NLHI8QhuX8ZuNFCEQ19HWg0Uv7kX7ghRmcns1cdIfEqZimseWcp9Fh59b38+PyPbF+dkp/+4Pt3/+3u/w0P5O1OMdCGe6EEtl5iZ88B1Z2xPxVgChgUOFf28h9Ejb6sDXUX7jGo/TtTvicaGfczYf9L2RiMAr+e1jegIGHwSlbGYcHAicmGs/zAOoGEWJTIrc/433IGhPYsuV78Z0q4Ghb30Qm1/3fqTnNi51u4xiBkZoRIpP1d1dkvLPAQTVoIWpZB0LPvpq1Dl1oQJc8qa34rHf70NuWwSVnOmCebLu3LVThT+nnIvW6HymvDO9IZRUBxlARy4uox2vV6AK7T7TSUOsUwkdxroHHIfpwA5mLGQv8exhROSIjwUjI4rKjIZKT1kvp5lq07mBdTEPPJYTbIdERCAgiOFVWWzHqD+udkkY8XQalQp7vTUMnDSEjmP68Mh9P7FIQ9Sb7RWX9YjcMEdpZWpL8zue8lb/cqEsWbUG/YvW4sDt21GpxFDImWEdSRbbtuxCe0eHShOiypOTMwIAdUjI8tV6+Hz+smGlY4WqbE9RJJLvNhR7Ww4f4PuzfGCqPDw0JE41gSebD2TPXGmrR9ndIC0Dy1ivRtDRYS0i9qNVwpDdRkxBLUT7/VxG1YoRghTN5VkFHTSck8T+P4arOOeqc7Bj15M24REUY3BihVbakbxv3sb1KPH8+bj+G5+/ce2zTE7n8defvRulbC+iySHEO3oQTqTkq+XZWsQseD28JyySWDaICPpY+1pRoYSMuk3ATcpThjeSi4kDovUglJPbtxmiduSliepO4cHL8ubbjFKsaZliqLZxvUfJ+Pyg31ecjp4Pvhlbz34rytN5xL/0Djx04ycxVA+QDMJymHy+K8SR3+3TPP9J9LCCAGORBvrf83IUExFc+sYbsWdzGeV9wPjeaZRmK4riTDX52fI5yt2sXzjf8Iv9OuPb1sQlNufAqA4RXn+jWlebhwuMt49kACO/N5Ei4YLvx1kvmixvaHKj2kBnZ7tmACnFdQtSelJuQIrtOTLDeQlzCh+7SBwh4iWbirp8RhRjiBLJGpqzY81Ct2tJB5acuxz33v4ztLdnMDY+qgXPQ0GIrwO1rN6k+39R94F1KOvyxWuPx4LFq7Htrl2IluOoV62VNDtDA3Nayc6qFqQgpFLiPNy8XE7URZiHgTDWx2XH49a72kQlJFPcyA6s0wRHZiFFHXgExej04QeS0xHD/L8ccUezhoydxmyF7SYjuqS12AlAGYWXkk6T+lk5ZWNMxCngoPZy3oz2SfaAlYTm11xGOJpANZHDy996MXbu24QIsQcX/US6cIezJknOYz/N7YZ5GamPrnPMKR7dQQQ1FPH+z96CHaXFaKQ7kWrrRiKTpZWh8ebFt7Y51fy83LBSvIt33kLo0bY1AReAPoAmk5nxFT8db4D6qM7sjQuGkUX1kRM4z31YZ6XJn+F8VR8RWf36ekfpgbtQcoz5+/igC11JLL//G/jjyW9BtJxD+IPX4OEf/QLdG3chQ1mRU8b4lMPD/fNTEJ+O8waRZjlD5PDqM3HBh/8WhcMRjG2tojLZwNRYDqV8WVRJ/n5DM9lTY9O+qEXNjapF5IyxCckTxWUNZKQLDgbjTB2SPuhRZaATWxncAOIic8GyHUGgq16FbFZLrHfTKBbzyGTpF30kjWMPkveG70WKKP/Mz9Pf34NKuYAoxeHsSTtpmmHJHnCiEiYudlS2pxvVSBVrL1+Lu371X2gFRW1wwzCIskfmNq5q2WTWMopwBFXW4/1DOP3sl2HTHc8iXWhHhZMWNfeX0+Zz+r6JiRkd7FR9FQrcPBmMTdA10iOwbuCb0n5D7bmB1FJEQ77RJPHMIa+thq6V6DyRaNXicqkwxp0FFjusxQtw3lwUshcLeSxZskQOHbn8rNJrk05yE9YklhH45gCtufQcRkll1pRMpw055gFCgCybQTKdwLpXrEQtWUJuclxRzrO45rfT5kfU+evyhTa0slRRJFvYO1HEez/3e+RTvYi0DyLe3ql7yhGyxEq4z3h4kdg0V5p6A0K2g7Rx5/UhFcHCIWRSWecAAelpmRtKl8qr89P0XJTWLRU5w/yAaChmG5eGcZY2zQey3BGoTaCaJhxC/+PfxrPv+ypCv38Q1QtPRLBgEDs//210BMa+YVrpU/T5ULscMlzNoNRHtUqA0fY0rnz4R5gd48jIJqpTZRTzDVQKNREt1CYi4lksoFY1hJu12dT0jOor1U6OTEHqHxegro3v3wo0c4c3lRan/ABsu5ClxZ9tb8/KwzebSqPM6X01MxqjQKEldhI5zDVkM6aCUZSNmhOEDkeqfep1ETJo2VKv0nM4g0hg/VF7mWeT6JMNglQsTyJo6+1BEAuw6IIleOD3t6NQ2Kvszpz3HVVQLRhLr8jt5ufN53JoBlG89MqrsfvRPQgOhjXcKyAWI+8t/r4wxsYPC9hjxC2WCxJ412stkNQhOicJDorkloILMkuQfEJDd0YOpsI1lUk84HhPNc5FKbbp0KSskh1QXFHUDhbbuEqXiTxLFM9B3swSOJmPkZTCBJI76PJovWndI9fnV8bnhpyTK82+uRhbLtXUNQZN9A72IhXN4GB4B172hguxY8dmtBzpQp/BaafnJZxzSL3/2p/auBHSGMMVvOPDP8b+6hCa9NNuX8j+lAbhRTkyJWjo+UsUYnwoHboq4R3fPPTH7vU2rc/3TENAxk2Q583wqiBvVmBpsOtpsYaRhzKRX9azCVQd2VunrzyUjzT2+TVvS6NI7m1IEKDntn/C7L5RTNzwj5g5pgMj734z7r/qnWgTTzo8x31W9J6nyODpJ80sca5mCJF4EqUVwzjz11/FzLZZjG2rojhdQatCTjLmVEBs4NuDYl1IrS3TVqKGxtFmCspNw542U2qe7qxPeRdZs1k5HUYg72SysxpAqIae3m7r04aZ7jRRnM2jUa3pfYylY4boXNyVUh4dnR2OWM8WEAEu1q0G5hABZcRhFGcqVy1NC+Biaklmm998rMslzaRRWob0wRgGTxnC/smD2L3lXsR4T0oF0fz0DIRZmFhE7k9BIMLDqRdcgsl9VcxunEWrGUWjbtkXgSd+D+8Jx2hOTZLOmEalYdI5sqyYqXhnR16bZ+MxSjEFZ9sm7GprRdGgrpqfhndsLdFjir+D2YznePv2ju/zsg7394UKNQKWTCWJzAqoi1prrZgnSYTtS5YxBMmsDWb9X6uVNamwRc6xMayYXbFXnMok0dPXp2wzlIwhtSyEodX92P3cs3P7lHdlPt1RmZ+TnM7fzD4jnL+ZqRLPlRt404duRS3eA3QNIdnVg1DELHk1b5qqrXIVFWpxnTrPPMiNjCRA74mudQFbPV5/amSAiJBQf8IJineWH1IJemDDzWxlOpJmisOer+PB+hPHD13yOb5aTc7RXmCJJHlNRD/yJvS84hxsPfU6zCYaiH36emy89kNoZ/3BZhPbDO4OzHfNI9fYUENu8Dj63/QqLP/oDRj940HMHGihNhMgny+JylatmBsDwThGByMNkAVNdJgLs67emYjqqseddIw31AEDAnpkpm10vHTMFod6oFHjMGeyaU2J54FWzOWRcgQNtUGcn5babBznQXJHMinU2ZBGigxicswgiKWSLmILktTPUiWPVMKQZ1uMRkLhwoln0sj29yGZaUMuMYv+lSPY8OCdKBbH0Qz53nDY+pVCV9kXjqKrqw+9CxdjyYqTsfv2XWiWIqg2WC4YEBONxJUm+tJm755RFIs1AWIqNajGd3Wn6WTtsOZPa+qiy6zI4ZKsjiUH6+NqUbUpD1HyibWhdIBSxGLiDF8CMZVmr5UgV1+fs/LhweOnHaCltptlFWzVmeWrMees9UPChge4uI6Z+VCEQracX/8dnW3ydeYG6h4YQD40gzXnL8Xk7CgK+cIc3/7/tkGP/rf5GSIPi4/+8y+x8XAK9WQPIv1LkcykEAlbf5sBgPpgkZ44MJ3llLMx9k4hyoofyq4ShMyaw99Unpysz+RqSEcEWY2YKsdL/GxhM4Pmmc3hTil9wdtk2oNjjLf+rU9plULzEHCT+PRQww1UXnseFr7rWmw++TpUQhXkPvQa7P7YN9Cey6MrnJS21r/mQBqCBOoXEqKOY/1Nf4vsay/B3sf3ojya4GhTFKermnvKVJAkAfZR9dlbgU1g1xhMmyJYoZdVJGY6Wk0WbJlxma7bXAVlqeMWgozO6GZYMmolPaVYLDdaDSTTUd2PGGvuitVpOvwcOV2gX5MAldH9eAncHOSB9/Z029eUHpqti6w6xVclH7hoKiHH8GKKzjIm3dmOZFc3IskUplqTWH/Zi3HPz25FMxhFHeYVrc3EfrUDClMZaqtDuOBVV+K5329FZDYjsnyrboohEVuoruKCcnYt+/eNoVZpIXC8YJYUHELNtJb9XRJY2BbiRbOG5DPnPeW0Pt4n8pmjHGdDQbyTQpoai5pgI2NISJBg5DYLVqbevF4OaWPrTAIQaZ15z00QQw6zhAt0Z9H9s/6nJ7wwhbbpBWZFxI3MDS4mnzNnZ4eAJ0b/YD8yvR3ItrdjOnQIa89dhmc3bTK85ihgdn5Enb9Jj3z9SHmTL5bxtg//GuVIFxrt3Yhr4yYRallbj59NGAvLDreRVWaaBGpOlRb6Q/a4INwMxHAhsVtjDtwbWI/NHDD8KardzsqFUdgJ23lj2K8VgVxjJU1+NHcRrhnvEWBGT5uT6njGYaD4kuNwzD++BxvOeBsirQam3/NK7PjBr5B+bqeIGElK4o8iYjDZI8OnFo7good/jOnuXow9th+NQ6y/6qiWKJCvKYKZyDqEsbEJRa9MOotcPj/3wLiwGFIqdSpSDBDwNa2RFdiftHTQj4vkwZRxSKoiIiN5g86FIRQqeWRSSU0baDW4cAsiVGh4meprHoYG8vFwjEu5VENXV4csVxhdpL7yWYbIB25iBA3Q6JkrMQhTRANguob65bEc72hDvlnB6kvXY+NtT2K29hRKTdO+MrJwceZzeRNJhBN48aWXYXpvE9UdVQTNxBwrjNnXxMQEUumskUTC5B/PYuzwLGZmiA6b+6OymCjdUdiSMqSejDMePJRCclPQ7jYSbpj3kxsKRyIE570QFGP7i71vWcs6yx4Oqg61YqiRvNHeISdPKqlIE7RgYmUSnxXpq+0d7Sa0JzPKbQCapPMmcrPz655oowO71ZS5O1Vb/LuZEpSwZOlSSnWQ6uhCRz9/bx1d6yJIdWawc9s2M2dwr/nkIGPwuTrd1aN8fja0PYZGqIgf3vIAfnrfNFqJbqB/EVLd/WrFeYop12mZg+LqbJkRvTVWm2+1WXkUIHR/emVAhDTLiMkERpvP0dJc7UtChbXx3UtpGsGKQBFCFDU5CtjPqz/riezzkGRFXg/Pe8E9iRocYbl8GMM//gSeeek7kZ7OI3fNOXh28yZEf/MQkty41CTOO+l4AfT7zQ8P4OX3fg+VYgj7Nk6iORtFpWhuG6V8UXUaWU2cK0qQibYoBw4cUF0Vo4Y0n3N0RAOomkEIuTxTKBNu8/uJ9Eqe6MoA7h9S74g2p2nQzUhCgCkW0UR2kQUoJ1R0toOPQAgb/7EwXS+Y1vMmEtU1twdyFbt7ekVW4Mb21EDWfOLSSs3N1LAJpZxBzTjBXIAuemZ7OpFqzyLd04uZWhHHvXw1Nv12B3YfvgfhjPVVjW5qjDA+i1K+hD+77u147padCNdZY7PGZAlhdZw43rwCN1FgapKSvxomxvOIOg8ylVQsr9wi05S5OMdC5uSzxfvOdg9TwGQyjmicQ62LaO+JINsRR7wjBLb+YwkbyOXBrWqJnOwQ8lNljO8sIKjE0ZHtEoLPZ8MsTx5ebl3E4sYnlxJKHHlnbyNKI0UiVuMqnachBANGMT+nhOOa4ubPtmUR5yjObArJ9iw62zqwv7ATJ1+4FvtG96FW4oxae70Qq0+HrV+rag2xjRpDNWjgmnd+C7nwIKJdi5AYWoBwOmsB0GU0co7kYcyfbzAzkPRBb2dSTPtz6IHscUFc7o5E6szIWoOU1OwmeZ6nnvOfFVDBm2FvQhTZ80WYemiPUq6mVMcTrT04xVPyyER6r93VCcULWzSIgdv/BU9e8T50Pr0XB4fbUb7qRdj7ia+jB3EkXQtANiNKm0KIrT4WZ932PUwcmsL45gaCfBPl2QIKlQC1EoEd1l8t0TW5mJg+8b/9/f3Yv3+/wCC2BKjh9QcNPYRmczZwWYR1Z9BNhNTYYIZa8qWay5P9pQnmQC/WYmHQrpbkCD4QuTbWyygUaPNZ0MZRKhgmAk35Wgr93YP6XUoJo9bP5f3V/ReHmMWujafsaqerZkk6WRrmqSInMb+nC+muNqS6ejFZnMGqy1Zj6x2j2Hv4IbSSs4rMSiFpuCePYfkE4pVvvAEbfrgD0RBrSBJcmMITLDGmGK1x1Gar1zE6SmF5HHkSMlxfWCm02xCGYVgLkJuQBxZ/doajRUJVdPSEcPJpK1FJHha6ykgd1JnCsuZnVmStOLskO5RIl6zWSggV4sjtD9CcjSPCodk6LA2TMRqkyfr4u3mdbKsxS+Kf5UDikHhGZ6EWnK5YKQv152Zgq4n3PNOWVV86mY0h0zOIbNaR/kca6Fnajp2bDagSc3deFjg/w5y/cWkvzOf0wB934rPffhiNRA/ifcuRHBxBjPOZKXap1hR1fe+WtbtIR9q4NvpGskQCoXzuj7avkVmcB0Y09pD/88Zc3MBC4MypkOCTX9BJkbINJZ1Le90i8uGdC1hfcj1Hf1IJn3Xu7GFuhs4khv7wTTz7l19A4vd/RK09jpn3X46n3vFxLAyldcqKG8rFhhbazj8DZ9z8BRx8egwz2zn2gkSHGiqFskgObF2w1tKUPFqQcpaNc+XgZzAksSUHP8q0eFp7WRcjhTX46WVsKhf2CT0QRP6sjdZk7WtqE25GpuIkSgTNKtCsYHziIA6P7UGrSVqj8Y45aEwAl0tvfUrOKMrabu2q1Wgj9Y0T72KMTsyE3Oneagjt5M8kOduoMEOSI6wCJEDZj0gmgUxnP6ZLU1j1yrV47rY9KNXHsO3QHxRJGPHiSeqAC+aK2DaIc/7s1dj0o902uM1EgIhFDeXkM5+cnhJnmKf9nl0HEQRR1fUc68Lv8SojXwpR2ULQJxRuoZDLo9IoAdESzrp0MULxCkplTp8iDdR5kSkS2ybTjB+3YjSF0bVodM81qK1FwB6TW8qY3E2ZZVqZUyxpkxRMKBHRKBJbm6wbmyIwZNNJJ6yvzE1SUKrfqAgk0+cPWujs7taG5AbOdLQj2dmGTCqB8doMjjt7IZ579hmNnqFAgPZItomPjI19XmboWqHEC97+ke9hX6EDQXYAyZ5FSPQPWztP9jQ2zbBJphRH68kS2Ea3KrJz/zmaqOZXsR1kIdhefuMaN9hFUaalHIdAXqy4x4Ta06hpSp27za6O9Tm+P32YJvq2j1hNDlnVUe+yb6J6QTqKkYe/i22fuxn43h1oRAIU3nkp7rvpC1gUTyJFCy1ukgBof+mZOONHn8eWJ/ZgZnMIyHMKm03N0wgWWo06ckc6lTErFkYFprqMUAJ7rN/IBzo9M6u0j0R9LhS5J4gDTEvVrDY9oTZTvxiSy0WnVlmIJQIwPT0htLRWmcGh0e2oVui95LW6jkTChe7wAuPz2n2XKknjWCxapBMJ9HR0YXhgELFIco622Nne7iRm9pQ4lDpUr6LJD9BsoWfBEOIEOtJZlFHGsouPx7Zf7UEQrmDz4TvcLFoqT0Jq+fF6lq04ESPL1uPZn+zQac5+bCQes7k/DsvgY+JG172aLiJoRjE9My0JGg8btnr881YrTBGdhJUois0pLF2TwfAxMc3z5UahAGV2pqCNSnosQTmLKMYFsJ1gA+CYYfH9GX0kDuB8JqWTAcLVAPs2ziJR7UciltIJyufFSMu0XVkUsQoZHJCBZsoqK/NsM7PmJ/PMwDSzE+7o7tThlU6l0N7TrZSZh108nUF8pIH24Qx2bNtCtficc+XcBvKbeN4XeKgWKlW89m/+E610F0Idi9A2tBiRjB3CygxbTdkJMftgYOLn8BvX6lsCwQZe6faQq+zLUAJGXLB82QLz99CRLxh9CdK4ERGs0bRx/ffN5w97JZDoeTbvVfWFK+C5AX1KxHQp2p5G3wPfxN5v/BzVL94ix4vZl6/HQw/ei+HRKYFT5PDGertx0dO3Ye+zh3DgAQ6RLsn9QRPxOHCMzm9y5LNeq6HFjIaOteX+K3MA+hvXaihQuscSAUynTaxsfWabycpFxZRKG52nvqNqEgCxYV4VFArTGJvcjlxuDNFoSbUsDztzEfRAHVHmhA4Wk8+ZWJ7fx9Tf92WZsnGLE7Q5cc16dLZ3akGypJnjG3OiTSyCSiEn21ue0D0jQ4gmE8j29qIYKmHx+Wvx3M93Ip2O49GdP3KsI0r1HJMpaOHMcy5Ftd6OQ/dMqHXDe0ItrMBHaYCr+p1cXASYcrkKWk2OSikgqhLESP1il7l5wXx/orV9I0n0rS6jgSI48jrOrENItKWEPH4YSTWyhemiq+FMRWZtMHlVsf1IYwORNzjIyonvqWEsAwefmUayMoz2bLvUXRp/wllURLSdeICfrVLMI8t+OAUJ1G0X8m58qm1c/wwSqaTKF9a7HD+aaMugb3gQyXQbirEpLFzfh63btiFoENC0XNmDt3PRd97GpQ/yb+7agH+9dRciqXbEB1Yh0z+MkMa2WgYrT2sGQpJeqBSThxZXvG1UlbH+0OFvZTvI/1IPHPmNqwPI1Vi+t0nXRAIc6q85frLjSgoplkcuh/w5SF/hqNFU2id82zevmQp4PW2oiURPL3oe+Bq2f/6HCH3ndpHQ92YD5M9YhsKtv0M2mkAmlMBFj/wE5e5hPPGzLajnaa5dUCQ1T+SQasbZmVn93YvGreHvMwNbENq4nMlKI+1GQ/pgO+VN86g00bHImKKz7ufi1YPhYGMuxXACjWYVk9NPY+GiCvbtGsXE5AxCQVI/y2nsJHZQKKD3axmaHo8yRbQ+qWxjqVt1Nj38rASkGOXVKmsEOH7ZSiweWYQ0hQCKGrZYWKuaTM1cR9p7u0V5pMKkGqth6QUnYNOtO1VH7pq5DQ06BfIwSiScD1OAi175emx+chTl7UzVLavhYiLoM3/zkp9D5PHRVAAAIABJREFUp4tcvozpmYLmB0UTJikUGUGWrNaLrdfLGDwmgcXHN1DWfbU+Kj8r2WNjhw/bHF5NKgirPqbeli/2a/nypQzfmwyzYjGnTcwoqbajyjP6UYeQL06hsD2EcKFPw9nZzlLa67jEnhxRyuc0nEwRu1EXXTKdsdGnxFlY5tS5bqIxOW0wE+jq7UE8k0I004FkNoV0RxI9x0Yx1SphanTP/x5xRROu4/K3/Qtq6aVItfUjGFyJNg6n1oFYM3koe7bMwOTNZg40Kj/dxtWh7sBiZbX3pldwjTk5mZ8DyzEVBjSJ5jh34+tIsX5xUZmb0TNSlKI69UlEnEurYUXgTiT1gVpMK72W11EndVqFm4iuWobBX/4znv2LTwH3PcUGHKZTLTSuvxjPfeZrGEAaS//i1Vj7ib/Dk7dtRTCW0DhGtgE98drX2uS8au4YUVPnhC/k1dXjBKV4itPxr8wp8tU6pmdmdMKSlEEiBvusTBvVxxRbxaKELTQ+3Aha9SriqZ1YsaaKeKgs6h37wKGA9izk+LaQmy0hXwyjVGggN0NeM5HmrJwWuAClG43aOErdC01+sPmxjBocaBbUW1i3fDWWjyxR+nZk0XOBh1Auzmozd/b3ItPdhRBTxUQDx1y43m3cKLaP/xahFIeQtaHWIEhnM3hect4VeO7RA2jujaDJFoizH6J4wlM+2XfloUX/KY7YlKkc6/95jCRiEDxsuB76FkcwuLLGjrMOAx70Skk1k7Y213vl/UxzfKfAIS/xc5xkN8VQ3YNoTBY86hfX6PVF0X1Rm61RrqERaaKVr2F8WxmpSj/SiXYdJH4kjieAsF7kpA4uPTL8GPm5cYlTELASPiFyjQFz6jzEY4hlUkhmOhGKhdHe3YtwZx4DJyzBto1PooEjE+xfqIfLzz86lsd1H/4ZWul+pDv60eo7Fl19vXNBguWD8AWJC1gyEFU2uazfuPwzywWBpAQA78uulJ28UkOnqVV6Ic8hywS0eF2Pljas6sM6cMk0kVxczieJKhcOfXL0LEYTpteqsWWK5rpg82xpIpEWkte+Ah0fuR5bTrsBsckZ2ZYcStTQ9o4r8PSnv4W2/n5c9eB/YirfwrbfjKFUrDvU1lJu/39t4oYhyXxgU5OTc5pbXrCoi06ozfEOpUpF/5eLgxBiM8uWVlOEdZvDyptpaDqtJAJUC3n0DBzE4iWHETTZNqmiPduN2Rxnu9L6xc+9iciZQumO0iCgVongyae24YktE+hsa8dLTlyNZokzm2i6xkyag5pJajBTOKLe0SCMM9Ycj4V9i0w8r/voiKxNa+/0DPQi2dWJVjSO1EAWg2eswDP/tVXSuP2FB5FvHNbnIPGgs7NLm/HMc67Apkf3IThI5NSyFAlF3JgSHrTcdIVCWQdaqVzTxuXfE1kDznjYJZIRTZUbGGlH/6pZBGSOEbRzNjOkKNKOtlgqOWNyox1y7dAi1jIih54T4XXmdj4bJGupq6vXlVvUKhtphob/nH/M2c5BuYXn7plAX2IREsk04gn1H8xtRAcmMDs95TjMpgcmWMcNzWyBXtcCKmNUxaXNtYMlA3vA2XYh1vE0dbMVLH/pWmx9+hm0wjalns4f86eRKKMTs7CFH/33g7j5rr2IJPsQ6xpEZuEKRElEqVudTR67zBVZvzpCkApW9YCspFBP33GWVXrdk12hjWtOFRSJ/x+q3gPMrqu6Hl/39f5m3vTRSBo1ywXZwtjGTVRjU0LiNIwJoYQQev0IBPhB4pAAST4IhCRAICEGG+OAMTYG3LtwwZZlW12W1aWRps+83u7/W2ufM9J/SD5Lo5n37rv3nH32XnvttawuYA3qT1pfixKV5cnqeZpsAfFLBAUCGX70jyAP0y0BWnEBWiJza7jawAcV2g4Uy+Qy6PvJlxA95wzsO/c96NRrKHebmE220HzF2Xj8jofwzs99Hqs+/Pu494YtyNX7MDs7pw+biLnUx2kVMT3Se1OKRKLYRn7n5vMsMNZJfAisfSkOzrqWI3yk+Rlf2EV/vpajPXo2D0+JRm0RgwOzGF9zXAymUqlPXrOdjk1+kDRP1Jd9S35e0tZMo7gpggGnkaq1Lr76P7fLKPwL73kjwghPd05MBRpW57V+/8e/QaXDnzcw7LLz1uOVZ12OgfQqaRTziymjSc+GIm+k+0uIZ3JIjuTQf8F67PjZDkXo/TObUQmPazGTkNKhtWqng0tfcw32PnMCtQP0ljWmE+vpxWpZ78kFz40eCeKYmpxVKsnsl6OQQeKUAiiJGcm+EGs3NrH2jHORTvVgenIOM9PWDuLaq5TLOn0LhTwGBtNohgsoV2cwuzCrYQRpKVMhgzy5bohMIq9WDlUvyN6SxxXLB9jAvjIWyQpZfcxUONpI4sAjMxgsrUSUcEKXabOVaKJHkuBQLUuQ3VRKzKmDLadMljW7lUNMlWXyJVO5KFJ5km8515xGN9LES996AXY+fQiRxFEzaydV8zRzavKyaVVCpdA/ec830UivQyw3gMTYOErLlqPO9daoqw2kCTKK2JGYQvqoJl7dUEVomIuxELl5Q2sx3ptbp0F6r92rGOXsG22HGVDlGSB2ctqN0Hcdw8hrTqmWc/Uv0zqefhKdc8HBc3XjolDyRnYQFNNYvvVGnHx6D+p/9i/oBB3Mtqs4HJRR789joieNq/78/TjzbZfh7m9tRzxizBzJvTruLxehGDzauB0QgeVJQRYUjckYnZleefkWP0RAqp4AKfYrG3WlRwYYtKVswd83MXduFPZ7O4iHc1ix5llE0EQ0QdkTU/zgzK6BUVZfhQTMmm2107woPE+raDqOaBjB577xE8SSSfzNu9+IpCiR5nNDKR3K3PzXzQ/iZNnsTshsu+jMcVx+znqMJS9AKk5dq1Ou6gzHHCLPDfUjwtq6P4mxTedh283b1O88PP8kZhp7RSM0CZ60FEAuedU1OLm/hoW9DDIEEdPiSUsxkzTMas3UBVtdTE/Noc2gU29ogJ7WQZzJjSXjuPT1L8OhF4+jPksYihmWTU3RGZDrSzpRBAqlwUzP4yi6USKolA3i4DiF4aLI9sVR6Ith2fgAqpjHwuKsergMoDZ6xwzOQDrvGJmnxGu9hlatgVwhg+fv3QtMZpDL5Di6b0olmkIyjyDOR3uZGxmQU5FycUGzy9zArMN9y04kf6LfuV75KEXjSTSjLVzy5xfj2YePoTA4gw4WbUjFtW6k5qF6NIqp+Rr+/JM/ALJrECn2Iz++FsXSICo10i0bQpLbbI+xdFFj2IzePFCJjuEztq6szmVPOLgnty5coiJSBcBN4jDdtU3vZ0g4V2cu8s4T04mWmdQIh925tOUMHolqlItvQJ6a+LkEMVwqJL6zHNhMiLozWMTIk9dj5ye+iZ5fP6M0bbZdw57OLCbjHWz86/dhaPnZOOOq83D3N7aj2XQ2iWpSGynd6kPjLbMm40YyTSiL0kJK2bedm1OdSAofa7I6c9MuKZI1JNNpjeNR0VHAgUAvOy1JqjCSxjxWLt+FZHIRrWYUuQFOA+WRTGfUP83mehFNZJBO9yr7Y13IMRi6tFcX64ghjliGtWRELCe2ctKdBTQW66g1FlCj189iGeW5OTzy9Db85I57ZF7Nh3nhmWfhsgsGUWyvwmB0tdH+2Hohw0Ynbg9S/b2Ip3KIDHHjvhTP/OgZtUcOzG5GkJmS1jQRWva42dIbHH05BkqrcODRE5qMKZV6dA/lseRmUHkP58sV1KpNVBumQ3zixKRQ+J6+IkZGR9BpdhGViiUXgpOl5TnRNXcBtZpEYjGt4yRdHUSMoLyNjYAyZaSSf5tjXKxDmzU0W1W9ZrY/iUIpg9JwEYt1utVzGiqJeres0oIpIu1EQ2pDLwZ46vbnMZQeRoQqjqfRD2WiJu451TaJ6prtjQbVSUmNccyx4MYKTRObP5BKskWk0I1OsovL330pnvjVIQyt6CJIT9n6s/PMiSMAnWaI791wF25+YBJBbgSx/mXoXbNGrSt2MiSNxIyGpZqo2wTbDFOSzahcPKxzQ5SZ2YLkkZg2/ya7Zmke11tlcjNQVd3zkvnJhXKx9RM3JQZtZweoKBrQfyhktGVLKYZcYMPm/B0Spjkpw8hlBlDOe1cnfQTtP7gMy771Gex52ftQoNdqq4WZTh1PN6YwE29g0yc/jGUbLsbKS1fhl998TqmkSahyTtY2rPVBjXLJZj5JFFww4lG7vi3THqV+buHyz3wYhOHpm0OgiictR/AUDNhCaNYQTSSNjJEJcfErVmLjRSvQbLOma+PAzqOYmSrbYqi2kE1R7yiKsGISI2wruGdvi4Slgzxnjb8svnA0wCInVeJAIhUjrVW2KDz5Vm8cR74/jlvuuBVbH30c73zrJrTngebBBPoLg0orOxq/o0VKEem+HgSJNFKrchi79GXYcv2zmk+eaD6GVnDSdMUEfzHA0cN3A8654GXY9ZvDGgDoKZEKSjc9Iu3W+uKpu0jt5BA4Mb2ogMfxPhp0jwwPq1TyShNauM4ki382BcdT+timEMLRSJOo1dQPMRCJCLS1WHUSaR6Vvd6YNhb1t6xWZX/TCctziAANRBIN5IeyGH/JEJK9EWQzaWx7bCdmtkxLWYLXRsCS7cLFhXkro2j1kiDLy/qlTFs54pchcpzJ6DPJc8qpXcTjedWstVYL+WVZXPSWS/HgzduxfLwH0b6jStm9bKtknniX2028/69/gD3TRQT5fsRH1mBo9Rqx3yQWWG/pXspbOogiSnIJcxAe2Jovpv2qqZ3QOoeaYzLvZqr8y8IaJnYGOBnp1eRZ+IA9nN4JDWRgFKTjHFUfqFPbpfdMW4oTnF2MDfSojxjtzaEQTSI9U0P6yDzyQQyZ0Oh8nJYRYubSbTbc+3/+VUSWj2HqlZ9Eu07fmTbqQRf3Vo/gZLyOc173Rlz+rvdiYMMI7v72riUShyhyTppVrCanC8XZUpLjBbjJb9a0hfiBiWJyQc7PmbcP6WgLC2XUm019Dr4IEWcutlazo9bJ+o0rcOEr12Pn9p0oT7YR1uyz8D6xnrUpIPZR3KA2g0eap7YRWtjvkxwz+7BqrDMTIbhmmQNH+iIa/TObDNZiXMwiM3YB8owi2QbGNyzD6PIUtu16DJV9DfQ0ep1nr0V61qaF/l40IlEsu3gtCmeuxrM3PC/q4Ynm4+jEp0BCCjdmtVpXxJ+e6cNVV/8+nr99vzIgyu+QX8xgJuRW3NgoFqpVIcknpucwMXEC685YJy0yotAqExRALYAQPPNkeNaf/BmpX4hsQH0rcortz7JpbZtesNZFp6PhD9OHMoUSOfYRXHIqFaT8MSgzh0uojWYHB9dUPbKAtRcMoHdlEQ/+zz0oZcfUZ1YJ1+miTMlcotSSCWIJY4rTTJ954kZiEW1czUDnrBwR6huhxnGAMBrFqgvHsebyjbj/hucwtiqD9OgJE7d3Jy7/w4EI+m9d8bb/RCs9jGh+AMnlZ2B0fBUqi2VNSzUrJA41jeevxUv2FGm6DFIdySJHui1RfMlhR9vLP3UR/CK3WuCU1Afk0yrPQWkKS1ep00a920UlaGO2WUMtao6g6jG5FpDVwaxnzDE9xqFrJz/C18h0I0hH4lgWy6IYSyIZOFUL1obpOMa2/xQnvvsrdL95q8TXNHoWAPdWD+FgtIqRM8/FH//Dl5AYyuOB/96j9IqRh5uL1iCGIFvN42VkZeLklPK5eQhQsX7jKcs2kLxuKhW1fCq1hhBlL1zOh8yNhxTw2qsuw/TCNKYOLjDJVeZgGAAtNHgfTLGQIgIqDQJrpnMhSfxM8q4mvcLvg4GuZSNyGgM0QREbCm93kJdReFe1T1xjbUSYOYETWtssE2LVOT1Ysb4f9/74HqzIjZpCIqCZ6Gwhg0RPH0YuW43U6Bieuv5ZpHIJzGIrgtSihvQjEdaslvJue66B93z0A3jy5h1OEzpts8Ed6kIvuuujvUkTEycn8cKBg1i5YqUc8lhSeN66XxPcnDa4buqNavE6FwquBbLYGJj5/IxH3LTZU4eV6BmmUkpdGWDJ95ZAmsdV2I5r2SY2qVQ+AzMm1ymnLKmJVryG5WeMYt+2HcjHU8jSYocGZa0mUlQa0VohN7uDRq2KTIZa14biExPgNTAQcu1Qj4xkmVQui3YnwDmvX4++1Wvw4I+fx/CqNJKDxxCJkmtl+lpm1cryMYZXX/t9hJkCYoUR5FavR09pQCCdKaOw5SeKn+mVc+M252XIztOWtX/A8kLpLenGxD4I7gYIbi2sNQKGEdzEveTGSQdxVBp1nIw2MUPurWmfIqmFazrKS9QqH2nc3KoYGC4lJkZtNa21g3JNYFVhAL2kqEUjSF16NoZ/+E/YecF7UVqwi+XTboQdPFQ/jF1hGcNr1uOaf/4yOuk0nrzloBucj6lWJW1Pin6sq2NuAH1m1lJXV/96aRJ+wkq1opOWNR75rVTTr1IeRsyVhtQQudHGx1cglyfnloPzMRmDeWCNlpj8ko4SaXpk/lDGhkqGFDjPZMXSkayqZFFtgJs1HE87vo6EzCUI7mw2Q0OOBYRJQTIuphI/n5/AIkKpzglqaIV1XPGnL8Hdt9yJlclRbf54NonSYB/i2SLGXn0m2ukinrphO4r9GXQKL6IRmTUiP/2EZNbVwCN3H8Sn/uFzeOymbSLJcAHnC1nmfTpxzUY1wHylhv0HDyFTKKK/t+TorhD/WYEukXQaWoH0vCxAsGb0AweGigpEdKZfAozcZJml1bwvMZlUe4cBgWP8+SXdaYNdrP3H2VjzI+Z1erBK/K92oB5rM9bC8rF+zJ84jqBu4JQyApVPtJupoZDPaprLanCzRhFTjWoc7CqEXeTTBcxUaMaWxiV/fj7CRAFb7ziEvtUpBPn9CAPTuxaCrtMTuOmOh/Hft02ikyogPbgCpTVnIBZJSGmDa4EIcocEmnaIUqKMT73zYmr4c1uIl0ywkyi2tTg7CIRykx4bR/BTlypbBW99pHYsgulWAye7RBQ7iMaZf5skqRBChzKfcuezgWu/kUm+9kg0R/y0yZkO8KO5k3ptugcr0j1YdtPfIXbeRhy76MMA7SzYL2XWGQUerR3B0+0ZpHoG8Bf//m9IFHvx9O0HNMequpbNcg0RGMVNoEcyKVcCetMI/HLWi0x/+Vl403jaNSnG5cTOadZEA2NTKAReuvFcRWIbAneKjhyyd2OJGtVzXGcJBzBLIXc28JaTMQRqBcXkfMfIzmvU5FWbC8ycFzhL7IcvpGLoSAeLTu+Zi1kpu9LqhkYBqeIhPayQChJlXPGOjXjqV5tR7GaQySbQt2wZYqkcVl25AdVYBntvPwwkO8itnEGQqinCN+pmvcF0+ZYfPo5PfflvsPmGbTqJiEzLoiNus7tSWIwncOjYBKZn57Fs2YgWNFVPSLThBhKRIpdRqqzhCfnzWFamckQePmyFcTCCxAn2N40vzp4xNyazHdmZuhYjf1dOeU6CVTI2ak2ZionNDTEUOxkl9z4aLHAcAa/X3ApaGD9zGXZvfwb9qbTKGvZ3tWkLBQ0MMIMiw4knLj8D8QKtd7WDOFAQQQsxNLvAa95/GbY/fxRzuwMMrouind4nK1jvrMjnVq038fYP/ztmo+uVJqfHxjG4Yo0OPa4JAlKScquW8fl3vQwvG+uIO9Fg6h62lIFxuJ7bivxslQPEyEnw4b/dnFsZ8g9cSBwYrkZDrHvbZYitHdQbzE9NY37vFMon5zF/YgadahOpTgTRkG5trCtNbiTmoHBrHDGNNOULJsWqCEnlokwITYRZR4YBlmUKeN2ztyGaKeLkBR+20SaiZ4yo0QDPYhr3LRxGJJnDO772TQysW4Hf/uQFq6NkMs0hAecWHo8rdSNowt6t6k+mZE7xgBtcZPZWG1XJmjBOVKXcwE1o1Lw2zn3JBs3JaqyRtbEYLWZHYsMFjHiWuhC8oOuA5lCDCGoV61OK8x2Eiqqsr0j14wnPoELAwtd7YpS5YMATRUqHyaRc5zTepRSqo0XE01ejctTI4uxmvSYXt3pzFle+/Xzse2gbcok0hlau4NGLtW96KSqdBHbfcRCNbhXFNQuIpG3OlvIpqhEjcdzw7fvwqX/6NB67cQcyqYxOWzKcpCXVaGB+gQGti207d2F85SrVf2mmyOKoW/+fG3ChPCc9KA1exE1czqfEGoUk6OQ44/LHZb3veMT+AGC5Jj4yyQgajjd5UgUtAotyBDRPJrUc9Xwc0EYJHefP5AXhWOZ5FZZmt4GRtf2YOXEAyRqrQ9P/5qnL0pmBk319BlnOVpMwoqEHBV1rMTYaETTjIV7zwU14/O79qE5EkBo+iVr4InKFJOI06kqYYTlBrGs+9FN0C8sQ61mJwqp1KPYPihE4s7CAVq2CwSzw1Q+8DJn2CbTCONLxAMTAqVbC9hL9mdJZYggkpjBL4MFH87Ikgp8Ux2Xr2YgAx8MOfrZ4FN/83idVGPuWrRCuIDBt5GaI+vQiSqV+qSgsTM2ifGIOE3uOIqg1ETZa6Fa6CMj6cYbYUozgmzrDQyqusiJhsPzAoaeQ7EQxcf77VLtIwJORKBrBi9EKbp99Aa1YAtd88WtY/6rz8MD/7jRjKKKCBDlEljAgnqcAbzYfsCIaTwApVBhVkX+fmplCxGlmsd5imsxTPpVPo8h2Q3YQSal4nNa49yWA09vSInIOBamkqWtI3lSiZcY+4ukraRtOHXWMQM7711PgUD/5uMaE8WN9POW46TUiF1JQ3ZwHJCpXr5tmcYNlwYLb+AHm52dl07nxNWMI52dRjOQxtGI5EMthze9txGwZOHj/CTTDGlLLphGmKCzAUTe7H1y4P/nuw/joVz+BR37wHLLprMTuuIj5fjK5rlYxOTktOfO+npIR+cW+Ms1iZg9ybjxlNKH767+I5PpTV9pU5CzTKlTgH21gqExBNUdrvSnrYEYSjeh05vvwuTVqRH1NsZGDHiLfcPrKPVcOlXgvKNl0KA03l0cFOtbL7TY2vmIcL255Gj3JgvkIxRMS4FP/v9NRz93PQiel1mElEnu99VYMYT7Apr98Be65YReCZgyxZXPYvvMxDA33Yu2atejr71cZdPzkDP74Qz9CmCshXhxFduUqlPoHUG1UsTA7j8FYG9/4wIVIR2fQiUYws9jGkRNtPPfCIew6SKFCUugIUBpDgt2JFf0xrFpWwoYzhxH8b2FlGOuEeDxawS/a0+jEUvj7D1yNs84Y1QcR/Y8JO2+6G5aWiTQb4lT/Y9Rr2Ywsv2RMz0b7QhURDq9X6xqs539bE1Uszs5hbnIarVoXlU4d1z21RQPhBza8G3EaLsWJ3AV6/ZOJDn4+sxfzAbDp7R/BVe+7Gvf8cDuChlERefrZ3GzDjMbI8W22NIvJjXSUw/Ipeseamj0jMvu4JBdwfnZuYUFXTV7uyjUrUSxkEDZ52kQEtFGrin1SBhyCNVJb0KQGbTVa9j3q/AaBshPV2JmMo4+aMZgZejnfYKZ/i/NLUbkupcmOGv5kJ8kLlptdDnu06UxaPRiYFUVNG54tphSqlZp0hDmFM1s7ij+59jIs7JpC34oxBPE81r75fBw7UcPhRybRDpoorJpBM2Kc5obkYUkLTeOOG7fiw1/5OH53024BbMWegtQReR1MVXnSHzh4CIOlQQwMDGj2laCeKW+a9BAXt3yg6EecMraVBTcT5OM94ee0oGHEDKua+Lma+gt7zWqjuNaM/68X92Pq6Gei6w3bmMr2XOeDypVEavi+Xk6HAUW1sPrJZhxebi3g1VdehD1PbhZYyFQ5kTCROZUmEjKI6bkxW/MsQQFFiRwGzhjA+is34K4bdiEVTWLDVSW02mZETtYdA8Tc3Dweefx5fOE/70c30YPk4Cr0rlqHbD6DykIVuWgb33jfBszMTeF719+NPQu9aq12wizaLEVpGs5eD0k/ThPbm7tFKHbAdPq7uWXhb4MKHuLoFf1fIgE2jPfh/33kLeJZsk9IXS8lJBQN4/51Y2Q8+ZQGM/+P2ryrTXU4epYgU1pTcrFTQZFN96a0rchSIkXs9X/xWcQjOew+511IEYlNxkV2JwVsPt7FLdN7MB22sOrS1+Gd//Jp3PPD5xFWYyIPqL4Vq6QriF8mXS7FJLrMyMnWglQWnFUj02VOBFFqhbS+voE+jA70C43W4IAAD6tXKA2zxBJzJ6k3h2ZU5wJhb5btDqZ+THH9VI8GviWMZ20I9ZmdGsPC/KLSSvYbGeGloOioLkojvRgd0XOaPXMYvV4XGGfpvpFeOBNbq1ZQayziirechcb+eYyuWCVdzHV/eD4OHC3jhfuOotibRXr5CTSCOSG4YbuCarmG3r5+/OJHz+GDX/4YnvrJbqSTGfV8+/t7tQhZA56cncKhFw6jVOzVxpV3UoIgVsbKAVd+SPliadzRgpa8kJxgAfWrubl438yDmcGTQw8mSqBa2pVs2szOo9dcDttLhtu+zcTPLyqg0mMius490p2cDBjKxpzDngJMB1iszGGhMY+RoRCxWhcl9q2jduJ6mx1mEjIoo6+U27wMVJVGC2tfsQ6j563GPT/ei77eHoxdyL40Mw5qaidVcbc7EXz2S9/Bnb+bRJAZQmpsLfpXr5a4QHl6Du96wzjuuv1BHCxn0Y2aQAFT4EjUAoyoyQogRiVW1yEeQ8vZzqj99vO3vCn89+eewo7j80rReBrl48D/fu1TeohEUHliGY2R1WsEMTaDCc5EEppEKRX7kMwWjAXDiEqLCykXmJWJ0haCD+VF1Si84fVmFfFOB+e94VrEC33Y8ooPYHCyKlS7oxqpjXoigt/MvIiDYRmRvlH8zU3fxaN37kdnhhs3q7qT18wNzEXGB+4XjG/60+OGpywXDq+BYmDsPVebNSxbtgzFTEapsbxz2GoQsOK4yi6VVapKPqAUEu305P2gYiSV+WUKzjS909aG5EnFfpxqJKVwfsvMAAAgAElEQVTKrI8M9eSC6usr6d+46dRycEPTTN0ZeIiHCGGNxnTikTcrEQMnN0N63uz0jPF/K2VUqwvoWxdivNCLlWPr0GjGsOHai7H3wBwOPjqJUl8BtdwOpPIEQIDjR19AMplFqbcPv7hxBz78T5/Alpt3S962r6+oUUWO2c3Oz2F6fgZ9mX7kZE+yqDqcGQ1TN1E8eZKRZeXacX4+l6k4B+D5JZKFPIGdSbmb9eZn5Hog44nsNAZ31k/MMigqV6FwvVJjk9S1DWwAoszSvIWN3OxscwuHSNsJr00t72DLykh4oAZ1uTaH3qE4Tp7YjfHSiNJ/b5rOZ8uSRbJBZLWlqVNNSZsUFisVXPS2lyNa6MFjtx9E32ABwxvYozdRP1qqRoOkyspL3/ghLGIUieIo0ivWo3/VcnSbLRw7dAzh3CS6kSwiKQZz1sSWLfjxQ3M7sC9t0qXx19O+9+SN/xA+u/sgvvQfN1qNyRQ4AvzL59+PsZF+pAsFFOJ59GRzZq4cJOTnU919GIdvfRCpiRpirQCtiOkwsb4sNQIxbyS33WijFQvQoWp9xB6wTheO/kWjWP21jyJ5yfk4/NX/Ree/7kSE/jsBeZ6U34/hifljeCKYwUK1jU/98LtYrBWw73FaH9KuMo4ux8SoPEH5DzfMwM3Hv1MqlL0dyqUeP35cWkp8XYqDnH/ReZg/OYtChu0Mi+pSqHT1r2aTVSdZFjE3M6eNwpPGo5r8fjLJ09xmWEn898ytdov9R6NecjOSyUWQSX1OCagTOeSMqtV2xTz9hLpakETfuUm0gBIJnezeHlM9c0m+kjwxoxp0anYSzdgMXnXRWiwfWodqLcC5116MFw7NYebZBhKpCCZaD6MRziLoUG2pKetIBtX7f3kIH/rKJ7D5+q1IJTMYGh5AEJBAwpS4hrnZOfQVS0of5QoQYzCxe5FOmqQvN2ahmNMCkwome+y8p3QUiMdxgvO32gQcmrd/Y4uJwZZf1WrD8AgOs0fNq1g9cGk2n6I18Lmq3ylmElvipmjilTL9/LU5Kphel1h97FKwd85yo96U6+B8eRapUh25bheD2Z6l8sXPpMtrKZV0puP2XNkfvuKDV2L7jhkc3VHFslVFFFfPL302ri/yJCqtNl53zXUI08uRLC1HenwdSsOD6MxXsHPLVh0SsVQKMRcUlBI7PTYBul7uibO87A67coT1uqE51FW+6R/Dcq2Nj3/x69i06Qq87hWvxJrly5GqVTBz12/R2XscwZEpxJpdpCi3QhSWi0+9XIs0GrbvGOLpawJC2CJekwni9GHZ/mAkdjsXrW4bfVdegIF/+yxm7n8alQ98E22ieNTNZV4Ti+JAYx6/qh9CtQO89Qt/g/WbXosHfkiyAN+fpxJnNbnIynr4WuBy3DOJU/XhOmactFgpi0zx2t+7HJP7J5Gk8zd5xHSrkw2Iobka5eNwPRFOESVSSCVSJiymuo0zoQlDJWWBZLeTI4/8HUb/VDxp876UanGtEm8JyZ+VxpLukVH95mZmxDUmsslTtJAvGFgjw+cKkjJutv6lpYddCdNxU8zMTmO+OoU3v/4s9OeXoRWmsOGtl2D7zuNoHiZzDJio349uZEFpNgXIZ6Ym0Vfsx7anQ3zkKx/DIz96HoVsAcViFvk8gbEK9u55EaPLxjTN4wVEeL3SOdYEmPlIibXGvr3bbAqCTO2oXhE3v+AKaZMLiwqyslrRYL4NgdBPyRuGcXKKtaz6x+Q+M/X1/V63WW3w3U5gm5F2rbTTZIWZcUpUPWrcaG56Pj9+n6c7sYaZxTm0g2M4a3Q5MtGERu24ljzST2tSormsm0mznCrP4M2f+n384odb0F8cw9gZeXSyRzA5OYnJySnN15JnX2kA//i9R4H0CFL9K5EfPwO53iKObtuBxfl5pDJZxPjaMbo7OuNylRqm3qHzVlguZQad5KvLArXOeAo/f/t/hfmFNo7evwOTjzyDnmpHOsasW+Pqldqu91/EakwEnQLddnr6qQU+XG1cZy/CyMeWiixCNNnvcngLGvLabfVlcdbm76M9V8exqz5F2yGdtCzW20GI2XYdty7sxWzYwblvvApv+ZtP4/4f7bGBfuk/2QynGTTb4uHDZGvIs3EYwVmbd+MhNr35Amx9bCtKyX6zX6Qwmh6ODczzpDaFhLZR5UQggNo+PDG4qZge2khigGTKPVi1vgL1K0ny4O9wMUpkrWvADVM+LjKBTmxZKTW3jVivlDWr2kO+cSajFoiGxqVKccrSlEHSt4p4ijOVnjx5Agu1Gfz+G85BX2EE7SCNDW+5BFuePojudBKpeAwTzQfR7syZ92+jiXa9hhNHT2B+cgU+9o8fxb0/eAY9uQIy2Tj6+3oxMzuFWpmqjD3i+VqWxNPALCK1gLgpnCkVsw1D7g3x5896XjI/L0sE/js3r8Tb2PtlnSy/J1L6rBzj4mdgYGqr9hDnp52ihaW/RkYwn1pj6p1Od9XoJkkuRK3dz3gxRBJYTIaojmarjonpaVTbR9Gfi2Mk14NcIS91EqWstGXp7dW1skzgfHRQiuHyt70Kt3zndxgeGcNseyd+fuf1uPbaa5BMGn2SG/fhJ3bhB3fsR5AdRrJvBXI8cfuK2PrAQ0hn8qIFxxm4nfSP8AExv8wzyXVWrWRz3AdN5y0N1AQIHlp1WZgkYOEGdXkTk2SdRLqId4EW2xrgrKZXdDTNV40guRpQObgWIAegqV/rHP9MCnhJZ0onhtNf9qNK0WQC4w//B7rFAg5d/GEEtRYiBKjULgpQ6TRx59w+7A9rSA8N47M3/w8e+vkBdMuExTrIpvPaELIldBuDCLMhyTz1SGvsoN6u4aLXbMTBgweR7GTRqlcx0DfgVAbsQXHD+tqYf+fD4BfbD+w/q+6MUxzNUE2zrjSyvEYB6ffSqIs5RcoaU0WemN5xQMCDQ1RFPCM6TUmcRgP5bGZpookbeHzlSszNz6NDcoK4z+bB68GgmdkZG/RutzEzexLHThzDa16xEr25AQSJPM7+o4vw9O8OojObRC4dwzR+R9MPMdPKtQoa1TIWZhZw9IUiPvqlj+K+7z+JTCqHwaEeCabv3LsDq8fWIJUxQQKhuKSvpsxFnkGRQUci4uTyOkM4s/uwnrfpGlvQl8xrta6NwI0oUy4OprSYXvJpm9IF00ZmQCwzCGRqXWqEzwKcHywxhpJRHHkP/DXye2rPxR05hKi8K884LskMi1KxxEOIjs9WJ1DvnsBLhlcoaKaiCdXjXNK5QlG6VBymCNoRrL3yLORXDOPuG59D/8AIUkMHUGnPqvPAykrOjc06/vP6B/HYvgCR/DIkB1eiZ+U4svE4tj3xGHLFfs1gRwisatzTmQIwXXakFTk9SkbJdL90ODrZGpvkiyB4bOSCkLmzmQrZEc1tlzDW4lIU5QtJ7cJtUJv4M5sRRUSZe7kBYPVs7YubnI10bmhX3ToFgq7QaS7ske99FomLN+C5V38C2dmKgCARyAhUBQEemj+A59pzIof87a034unHJtE8mUWM9Q0nPNwQv1BhN963JGcTUrWxgqF1vQou8WYcsUQMhVxRtZTUPdyDZxTnBuHn5GmXSZPGZ20HnsBcOPwfr5kbyMQHyCWmf2qIYq6gHrMWdYcSLaS3LeqGciaYwUS9RYeAsg/LB2MuCHZ3fCosAbFuF7lMdqm9UXdzmyZqXlcdTDS2Vq9gfn4ar9y0GrlkEalsEev/6ELcf9cOYD6K5csHMRt5TlRJ8bbpbM/yodXBw/dO4+Of+wgevWkr0tmsfIlypTw2P/woXnLWOTZQTkIGTzFxj01xUKqMGiC36yZQaIi6Dbir1SNPZDt5xc12JwzLCdbTzBjUI03EBdBQmpWL0p/U8qJyLR1OMhmvm5vEXlM4iAsMzIJ4TRL386m8a2fa9BjUGzUKp1F8mTpPLUwjPdBBs3wCq3IjKknYseDPkPvNjIKOgCQcXfiXl+PI4TpeeGoSgyPDSI3slN4VT3c+V5VkzTr+4Tu/xY5JttPHkBhZjaHxlTiwbZumzRKZvKi2HDf0paWBbJY58rqYbfK+MEX3AVL9ZMe00+bVxnUnqMwTnAh1zGECPpIpHQmApEvd/MZUX46ImtIka6X4o15725v8OtaPT1/VdHepTPHj16D3L6/Gts9/F4W7n0eXyvOsYUTyCrG9MY2HascxG9bw0W99DdnhM7HjgSmZaVGs267B6hx+eN+096lvmKhj1dljqJ0gV5XSownzi2kwdbWRRQYWTaqIZ20ax5qPlCg4QRHbSOpZaqInKU4t68eeYo/olLJecWimVQx2Shjrpu5SLlNL5KkwMNinf7f3si//Hj7VXJxbRG9vr4CoQr6oIGR1HeVW6vqsrKXn5iawfl0By0dWIJZM49xrL8evbtmCYtCL/sEcFuO7KBJqI4bMJIjyV6t4+qkG/vBPr8azv96rdlCuJ4XesSzKxznwbm00qmbw3iiu63rtWZMRZpkJkXOr9atUzHQlk2rVGlH0viUQTlM6uieGMHswi5mMSpKWnaDKdCRiYJuXmAC/L0UMJ2jnUWX9V2xdu9c61V0KTZEEn0pzuoeKJJo4Yg8dXTHDphYn0QgP4yVDa5FLc+M6JJktwgQ7FnU0unW86TN/godu24OgkcHAaAnl+GOg7JJlXJZddFpVvO+6X6OaGEaydwXSy9aif2wUzz26Gf39A4ilMzppSSM1BQ4DvtgO4p89ocjfJ9IiPdXWmGGGnAdPLXu5Nq5OR9cz0kZw43Kn6lc7Rf3MrmDqUwerEFWfFnkyOVNE9TCdnIyG6ZneiN1k9R7TreKmjcj/5ycROVHBsT/4AkJasLuJGb7FyXYVt1b2Y7pbwUVv/j38+Ze+hF9/5xmErUByI0yrPEe1WOxR6snWij5kpIWL3nQODj5xDFE6kDurTJlTq/fLn+NpYO0ev1i5wRURXUnAFJjvIzUIjgemMzqdqVRhgZ8zk9YaUW2mE9k+nxHajVRB8gY3Ir9IuvCBj3PK3gyNi8UrU87NzGsUkWljJpMTpdOfSLZgu1goL2B6agIjQ1Gcf94GsZxecu2luPWm32Esvxz5YgTl+A50A+uVtrvUvapJA2pudhg9A8OYeHoGgwMDiOW7mJo9ieH8iGpQa8cwZbU2CVNWzchKLN1ojRokQFSsLvV/GVzabXMSiNiEFH+ezCWjjSY1tOExDwZHsqT4M5TvUYeAmAB72q5V5x3rBcy5AOrTaB0QmtKyUkQIshsEIW1QCDixBtrKMP0mv5oYAi06W00szM1gsvEiBrIJrBkYk2WNTjzO7VIzLR7H0IYhnP36C/Gr729Fqbcf/aM0VntCdS1benJdTGYwNXkC7/z8LxHmRhHvW47U8DgGR0ew9+ktKJJVxdOWjgsJTiNZhsD70GyTi2ClGfeSZwNKtsdbazqXS2WBW0Zfru3nj2058vEGOt1jc9WzNFoTREsypwR1bMSItYw0hAnXMy93spsEUsRNdv0ouRfoxvP/XQ+Q85lDJYze9w2kEgXsuewjoNUwwS+pOyBEA13cuLALk62qdJW/evdtuOfGPYg1yAv2UyVRpV48OUVamFtEtVvDm655FZ7Z/DyyyQwSbLS7E5k3SQU/f96JbJvyhbsXztBMCh1CJCmYVkY2m1MN6GsPDVArG7EbzM0t7eC2qX7wgVYWFxS1uWFtEZtIGiO737iq37xxmrtGKlTy/fj6DAILi1Wl3BxlPAWQUctpUdTHZHoeF23YgG4kjvPfuQn3/HwHBhJ9SOYC1DI7EEQoisfAydqwpfo5VTgXEweraB/rCkAZ3zCKY7snZNZlz6qjU4drgggwA5ykZyjy5nji0jB2QxzS+2Lv2g0fcMSEr8O61Zip1ttmj8bqO9akBgoKdCJgSe4320cJ07TW4LjqbFNT4cv4UT/7Hadppjcw6SANqstnmA4JnB5qOjM3Xrcx1BjcqTDZqDYwsXAUtfpRnLtmDfIpuiPwVEyimMuJQHTRuzYhjKVx1w1bsWzlOIL8EYTJSUQidr3iTXfaqHUDvOPTP0OQG0V0YBWKo+OIxUPMHJlAtm9AnRKbCIuKjimchLRWlWI2fMLRWj9wov3oWGgCsPT5Q9u4OgUdxO6lXsTY0H0I0abDPJFibl9fx0qmxrjBegAauHYCc6KuWWSkNaSLDEsnNL+/1CDniVssYPj2L6PS3499V30GqUqVk6+ajOjwwXY7uG1+L17sVNCMRPD3v7wJB7eHWDjYRk0Cb4YOU+jLZESZZDfwmj96FZ5/8lnkUgVNuzC4MLDwRlMwTSi0Nok9SC4e2o1ysRoZg4CKtSxIOuDgtcUt6znqlHdTLp7mp15mtQYuWHF9azWUeou6LvNqtTaG94IxQTbz1zVAoiPbDn5fPWNJqhiyXK/ZCKM15SOYm5s1KZhqBXPzM0gXFnHROeeh1uri5X/1Wtxx/e+wvGc50sUoKqltQMC+qaWq/Awc6B5ddwmeu/8wEtU8xjcOi0dbjPcYi8xbmDoqIe8zUXXSGvllFi0R3SNeL+WKfHvLVD5Dsxh13GbrRds9NwsWnqyUJDWgy6fdIrQwhXTaX+rLcrTSrRsCWkJYnTqkP5F4Xww45FqgTWdCyhFiWAmLYW+ZiLQJA+rnKB7XbGChXMbxyd1Yt6KEUjov76BcOidKJLOnTR+8Ant3nMSR58soUGu57wDaUng0NVQBYN0Odh+exRf+7QEE+VVIja5DaflqzE8fRqvaRLK3T9x5dll4/WQJ+iBH4pP65Kdlrr7T4Q9WtsqUHfP/nhq6QN5BYn84Lx+lYFKlt5tHaqLsIW0f6xdtusMI/qK2ufpORTSTNd93cv64Ek/jQ1JUMSKXAAYytXqyCN5xBXIf/DPsfc9XUdx2GKGrMcmkYozZPHsAT3RnpSzwse/+C7qFVdj36DxadfJjCSjZbCW/WLtcfNV52LF1J0ppRx7QWCEDvfWa2QKyFMsQZY+amqAYh7TrOiWLhaJtNvn/2KnK00AGWg0j2osUQMnXuBFBuCEqi1W1pPjgyfbhIjVE0NXMsjqpqHfL7wlkIpHekTG42LgZ/ICBwJ66aSHz9/h9gl8kQ1TrLczNTyGZncJF55yPVL6Is992Ee67/jkMl4aRzHTRzO9Bs0WXObsGRvf52VksO3MTnr3jKMbPXIG+oTwWDswikcqphSTwx1ExfW+T/GTW1MwseLKxx8375a1rFNYc51jZBck61YrWjW1cG7D3X6o36zZIUOrrXQpexAHIIdYGVWpLsoXJmfrSTkir62Dw2fN+SczeqbcYW40kDL+5DCBV8NagekcbmVRcDrdPTB7DzPx2XHDG2eZkkM4hmc0iSAa4/L2vxYO3bUdnIY7ScB/i/XvQCo07zo3rg/h/3nAXHtnZRrJnLaJDKzGy9gzs2vI4Sn0DiBd7FdxYz6ssEOEkpj5zwDlhmejBJta4R5bISjbUwnvpeRLBs6MXS3PK+wL5h8WXMHBF4PFSrcdvmK6ytoHzZ/HppRG0pUFMdUd56FqqpBNWEx2urcSGrUuXooko4meMYeDGr+DQz+9D4ut3oJUIbIiBvOVOB3vrM7i9ekA3+8Lfex2u/tsv4tH/3S+QhuR/EgsicdMzHjt7EEi2ML+/hnQuiUTEGFGGk9tMsdExzUTZQ+/sH9oYmRHjGQykc+TYTdrwrs3AB6bo6NJkntr8nAQ7uJDJhBK7hxGeSn6uByn5W6dgz3tNEoI3txapg7alAmH48MwHlq9LCmCrzkDH8bgWFhgcSPbnMECljoXyLMLISVx27gYUV4xi3ZvPxYPXb0OpNIBkpoV6ajc6odHzOBjBz0qlzNVnvxI//taD+PQ/vxeP/fQpFLI9qv3ls+PS/6UA59M0qydO8YOd+L0tNmOK8TPa6Wajn7z3XKD2/Lk2DMziZzMlDVsjptNt5RWvT1iHq/kM1OrqdbSAtTh58jeEa7B0s3LNnrMnZ3AjLAGObhSQPyHMgddIZYw2Qb46dh17DGsGSljZN4I412U8jdKaEi6+9hX45fe3Ih6hYF0PUNqNbruu4Rpz0ON67uJjf38zjpSTiBVWITG6BqvOWItdW55BaXgUAZlj5D+TlEIEmZvVMdKoeWYgccRQf5YFEac9zcNL/043DGJGAYKtIy8/JRbnTkneoBhrU4cE+5NCD1CkDIuYlmqae7g2tJN1JaTO2VprfViPkzef56wHVlg42AO1Af1EXwH9d/8rYtUu9r/hsyJ3sNdFyUve3JNhHbfM7kaVs4p9efzDnXfgwR/uQyZOXWVyUFvSpx1Y04uB0T6UJ+jDQqmUMvpKTP0c2OSmLeQzG7MmPReMQCWJiiVMnFojfM7KwguZuRPaVB1MTpWDF9x81BAyj1x7KP4UlxCBQ1k96YLXKxYPJYGc5QZrMVIifbrnF52eBetxPtBGS71QlgIsU7jJJyYmQLdDMoGmZvfglReci8L4CFZdcQ6e/PmLSNIwLdtGK/8iELAt09CDF4BDe8vsejzyqx141yf+EIc2T6gVR0BJ7BwnfSt0XsMbVOPIngZOmVay6XrZXK5lJ1zEhj1QRJ1fKgeEbVjqyr1FUIe/w03ja2Kesja/a6kjnw0BJVtHlk57tVCmzEKl5QYRA0XTddqTwdRsCzzk/WdQNVzFVFGMJmm5BK9loWxgGjf/8YXDSKcmsKa4BslsHKl4GmsvW491l2/EL777FDLZHEbGc6im9iDomqyqyeoyECziff/vFiyiB/He1YgNr5SiSKNcQaanF4l8QTRfL+fLtNnPWBN38Iw9May5lxzeYofOqUCnTb997NLQI1hEkj2rxxMqfCrp20I+yWFEYP/Nn2AOebBI1zUtYf2buzn8M8EQf9RbAmyRkUyeZUNDKP73p9A5ay12XPIh9FIbi0U8a0m2Gbot3HJyO04kO2iGdVx35x3Y8tAMwlmDzaS4H1vExks3YOaFGW0ioqZ8h9mZOZHmrTfm1SttzMu3I5jSSjZGd8gWmAm5mXyNMgbWbY5AwpuptFgqDVTEJ7BlWQi/eLIYD5kLlUHBojK9l7hYRNhfLKNUooyrnTys93p6Tuk6GzvLakL+TmWBKbLZiPhajekjpT752oeOPIerLtuIgTNXYPDiM/H4z3Yimy0gmW6gUzygul896oap53O079jJDI7snsc7Png1jj1xEulE2gUfA4P4VXWeQAwUlm055wtHDmDQ4joxYNBOTKs7Wb9aNqa6XrO1liG1HEXW+MWnnChIwOCz86eu3/Q8xetSyLDX8/8u7W6Bgk0paSylx9y8TlGS18UAGYtSY8oZRPOaXI3M+tK7O87MzePw7G9x9tBq9PYwkMbwpvf+HubbIZ781SH0DBWR7VtELXEMQViXtKwtGTLaGnj3Z3+GTqIfmcEzkBpbjemTxyTQx42bLPTYmJ6mfeLamL43K4MMch1cGaOSSlrShgdImCAwfWUNmm4feXl4qgi2qGSwtJvGcI1fqyu4QSxD0Wnj+r4Wu2yEzVpJdkrwxrHuM3DAjntLdwzU8GNUZGkN5IqIXv1ypD77V3juqk9gYLYhoriiI1sp3TYemD+AbcECupEQH/vRf6CDFTi0mT24kKIPeOklG/Di9gNIMd0KIwpCSkXCrto+kuVUe6PtLCdYn51Sm2AarDE0pb8eLLJUyNfmekpMs2ocjK8jX+BgudrmOn0NYQzQdhGfC4r3lAuaG5lUQ6tPTdJUJ4joeSbnygejf6OKQpVStTZULgvGtg3b8/e5IaSEz5Oi3cRiuY6F1hQuPWcIoy9Zhb7z1+PBm55BqYeDIh20Mnul9MCNR++g2mIFYTSFp5+aR7cM/NVn340dv9wlIkgu16P+NEE5kd4J7DEIOuKCyY8aCczKB/PbVe1GkobQ0oQGJnhSW2sLyOcKCmJ+Tla0x2x2qe+qk9hZ3XCteBMyOw1t8ovvytdMJ1Ogq55mmsnQ4sL3eINM2hg0TJOYJ7G3pzz9JNe6dVkin5ECcbWGQyc4mzyPlcOj4pxf/fE/wjNPHcXUoSb6B/oRG3oRYZScddbTxuASyFWp4z1fvBVBuojU0FmIJtNoR0IkMr3I9BQRTWfVnvHlmW1BZnYxE6B3Na31cO3z0J/JU3gpV2RYTATB7uWX+oPP0juS8qWImHNop+kpaac7cEWuB/Jk9U71tnT5u+rziQHiCnZaUbqJGp+WKgR4UEi1TQulbB4Lg1mM3fFvOPqVH6N962bz/KHyA8fx2i1sb81gc3NC0z1v/9cvYtXZr8JTP9uNdG8O6zesxuG9R3RTmIYnY0nN2JpfkW0QpkJyqKcJssbkLKAs8V4dWd1HdC4kXic3I3/HpFMa0olmmqcb7ni7ipCyhHSDCm5I3BQdrNerqB9ACLWsP93pLlTcUdx4GlEgTf1TaguTsU7pVf5OpS7wRWkfn4mUIpjutTA5PY9KdwEbz85j/CVrUdpwBn57yzbRGAv9ATrZF0z+1WlwVRfLCCNpPPrQBAYjWfzF378HT962HYl2QmqDYtPBTMD0rH0dq7TwNGacJqtaUr3wih0e+VTG0ek4i1XTRPZZhA+ACvSOJWSKkdbz5QnDTMfzc8mqUkakn3X2ma6OVr+eo6ZsIaq9ZKi9rlsaxca29wFTAcBlVabfXHNGajT/aqNaKWP/0d/h7BXLtH7e+sV34J5btiMV6UWxlEe3j8bW1F2O65mS+cZW4ez0At77d79AkMoimh1BrVHD0Mq1CHL9SHL6i1hL0vAWyxhs4yqbFe/aqJ3iO2jzdtGVbI2RMyRpIWvbLoLdY5cuORn4Rrnl7ZYGKyWkgqH3u3WbTm+oOsZACD4AzTA6cXR/QT5NUprqWiEmoO5qHd5URaEIYqU8Vt77bcw8sBUL190g7VsnbSTPmqPtMn5T2Y9y0MAbP/8hXHTlH+PuG7biyqs2Yd+Oo4iFEGXN4Hb2vCgVyjYCwR5OACUNBVwTb3QAACAASURBVBZTxdIbayNxkTjK2WnUQxMbM7IIPyNBEYmOU2vKjZx5fWhFezkeGEBC4gnvp05HTcLUMDg46OZ5rffosQJmAn7OV/e7YsLs2iDRmJ2ynHBp2YCBmDSRuGprkvZJAaSlRbnTwDkX5TA2MorSmWvwwM1bMTI0hHiuhjB3wG1cowmWFxYQRpJ46MHjOCM1inM2rcUZl16EF+7ag3KVxmj0ETIFCGPu0GjMaXA5Wqef3OF9phm2v07dM4chMHiaLA3rSjs9fGlgizO0ckjgyylfKqt5rT/MZ8ef4wZRf5ZC7sQiWM5wnJJ9Y4KhyugMe/FglzGv7NDxPV8/oWROF6HOH95v/l0Cdd0AR6cOIhudwdr1q3HFe9+Au36yE+lEHoWBJBKDvJfMTo3h5dtRB4+dxMe/fCei6TTiCTouVDEyfi6ifSMIqJsdT0i3mffJNqsRaLS33OGydDg60wD1fV1m1glNxlbFyu6xy2Wz6dnvYgG5WGARsKPepi0kk8Rc2pRehoQbXBMc5tInbWZPtnDRWUgjZTzZ4nBK9fwzazOeIkTQSvkChh7/Dqo7j2L2A9+0XJ7TKIyW7Q5muw3cVjuAxW4LL33HlXjt296HwexyPP6bXcgQhEmZUJdno4gho+a81Q6iw7m6kbWrXvi0TIJPXOkfb5T7XZIguEDYtuFDVt+NKQvTadce0qLUInR1BFt6ra5TyDCghikh081Oq24kFeatdFuv17UI1cAX5c9SS2YHZIEpqGh6hsCSSZuK/OECDBdQo9bA/OIC5soLuOLtG5GLhYiWhvDQT7diZNkoIqmT6KYOgw9eny/oyn40CJJ45rlpjAcrkUkmcOk1mxBms3jx1xOoo4pItItEGENIdQZZUHYQ7TozNUdL1MZjuuwGMvQZ2i2d1Nqg/kQ5je2kZ+ACuQKRo/rZgeG7ECxvjEHlBc2ZLtsYnAn4i4rqxAmWxvHcbDXXH19bBA43G670O8ZAaJJA3PAyg2sYgYanJw8RBt7JqWk8u+VuXPO+N+NlV7wcD/3sRbHC+saSqESft1ljR6Tgg2SgOnhsGp/8+p2IxTOI0Y4iFkHvygsR7+1Hh7PeZJLRtJxZmKWd+nzClVygs31oJ7F2JX/PeVOxzcl1J/R+z/JNp/IehxT7COVTItZporsJ6fPo8almsaKc4wsL0nZv6us3f4PVMA/ow5IU/Ywb2G5uG41uB8v7B1H4zT+hOVPD8WuvWxq3s/QOmGvV8IvafsxHWlh79cV4+0f/HlsfPILeZC+iEfbHDAkXgun6tdLn9Wn5Eo/YWhbyQfVyK6fxcDWvyeEAmkUXC0Zsd+LmYgZpUsoCgp/g8Owp3h+ioNXFiphRsiBh+8MRDKhW71Nj3ikuLO5BSqVaimj1Ne+3MaYog2qRWSqJAjSkD+vaSkTTG3rwi9VFnPfmcWRyUcxMtbHv8RMoDZQQpI6jGewz+F5JGXv0BDwCHDpYRW9lVMBNN9HBS990HgrLVmD3nftQmaUaYwJBzJU/zLAoYObKAx+whNTyfy7NzWSy+oy8h3SC8Pffja1YUD+dyHPa9JEvT5ip0AicbTCF09N+3nAS27Qee+Az47NgENSn5HpUIHTDIW6V83eNd22ZlhFvDPlWQHTWNvze0SOHMHxOGhe87gI8eOMOFHvyyA9XUYnss9aNzMpPHWS79h3DF75zP0BdKOIRuRzSw+chmu9FLEcNK27cuJzo6VniuQMKVk7myPxxA6XiKpe6xlPQHtAZbZs02Ltik1JlS1+WNrr+7ml9HjRQu8RB9aYaYVQvnzb7B8oTwvpN1nc6PV3236N8DE9Gr1xB1Hi4p4TBn34JtVQKU396HQLnym01UxQLrTpuLb+AmWQHF7/3arzkgj9A7UhWxHBq/LKSsVSsi2w2s+Rw5pFkf6O4WQmc8Ob4z6h0x/VVGY2LPTxhnU6wd2Vwo2QUaGMqafPHlkZazQTnWdRFf4lD8fYeZOH4E4DyJYywBvQYuYDXayoQnSWKHj+Hpm3o+sBUVSvXUmV+JZKkQrpB8m6AVDaDcrWMNVeNIozWcHxXGQefPYGh0UGEycPoRg6Ic8yNG+XIZtxE7SrTDVSOlBCPZZCkbUw2i9zqJM561UaUJ5vYvfkFBLWkVBl4DU2q7bsMw0zHHNWz01TdLz8mV9fq+p1mlB9/VOotewNPBNE2toXp5I7swCBK7Vp47nek6OgIPD4dt/64pY+MSQQM1cryPyuk36RX/X23zLGzJAdE8I3BVm1Luhh4NhuDcHYCG1+zEfddvwOFQgaF5VMod4/rkjWwIA65qaLs2HUU1/33g269A6WBMcQH1iOe70OHBtmprH6Hp2087daAH+tzhgOWevvDkWm8gZW6fxF/KAUIdoxcIuaUb9N4YMZQ5FPyofqg3KRuQkhC4K5G8RtXN9ydCL6INgc964fyQ/ovgjq8UaoJw1Ath95SCX3f/gSCdatw6PWfQqJtg/F6qEGA2UYZdy7sx/FUA+/73jcwfzyHZKtHahFcxAQZ1Bvk7zj4W5HX1ee8Po/kMoAwHVUEdEZT3pKT12u1sVHiuDgZufV9iZbbtBDracmKhAQ+TDyOBHUDUMzvxdIxN2rlepCkDfL7cQq7OxE73gu2pHif/KSJ+qcUQFetHrd5VV13c0kAT2qN7GV3A9TbC3jZn23Ai3v2oXqiiYkd82KlxQv7EUanjLhAxDcWaEiC6d7ciSlM76Xsar/xp1NZoy4mA/Ss6sP4xmUaQ6vXotj71CFUjs8h3o4DHZ6yvCd8RubiTqoFRQAJDPr6mOORzA70HGCnndYDw6ysVt2mk8gawSwG3axlE8qcLEngNYl+q6EGYytJh15kC1fDKkMhU6umZ677tZRJOdE5x5MXJuH48nwdM9kOsFit6NSWiigNrocyGDozhvv/bxcGh5ch0ks3yZrxn0m66YZuVrqNJ57Zj2/c9Fs0W1QETSJJadaBM5EoDSOeTCGayiKgeXgyBRYtTIE9wYbrm2uB18z+tIIz1w4F4pzwvxqSrssS7FnOGveUIJXfuKf/ly/CByFUWObXRqZYSkmcRrD6jS414c3kw6JQuPp6px/nLsbyPZQSqY61xTn89Q8iuPRlOPSGTyPXcmOCtO9otzCPJu6c34/Fnjiuu/NWbL5jL9JBj5QCeSOVUrgeIk2lWYP495WcqNNdVr2rVMren5uQ+lS+Ac5/07ifs+10B4K1Kpwxt5HuKXQW00A235ug1RKoFNhp7TeiT8WkHsJ6qlrR0IOXOl0qRVyNaKdGIIEzWb6I9GLfU3bkUkeiokRUCfxU81Vc/ofnY+fWgyjPVjC9awGZQgrJ3n0IIxxMMPUInrj5Ql4LfG5qAhM7ExjsWa9NyAkXm0VmfzSObjxALBVBcVUay8Z7kRjoRTpGzKOL6gJQmamgXWmhVWmjQqvQch1RyuxSmYQ92UxS/GaVMV0GNNNCZl0rE2s6CHAZkxK5pPllLTC/vvg81CEQJ4A1vu+XG+XWgoIBTHxG9P7VkL7zHGJ/l7PAqqdVG1Nvm1NLTlCO+obuvdXB4KQPSxwy/XozOOOSHvzmxi1YPj6Cbv556VJbu8okYw0TCbHrxZO47tu/QbPTFc85nutBduBshNmSAKsY0WZiAWSmxVNyP/AYAWEufg5+ziWlGAES1t9VOeJKFB1Ep29cf8r6k3aJLOFOTZNYNZ4rbxiNlJiqqLZxTCtLfE7l3F7027+mpQJ2CsoYiZQzUgMYvQCs+fjbkH7/n+C3V30UK8qGVMvXp93GRFjFXdVDaPQk8LXN92Pzz3ehlB50DB1rm0jIu1wG9YJ8veOjrrSgXL1gLQMzxubm42fSxpbVg33JOtJ5lRrybKm/r1dVL8m825zn/eSKofM8BZymFJlEro9NYopNv3A4gGbOXMhOtYH9YpeeG2pJdNrECHTiO/oogyhPNqZ3XOy9Pb1YqJWx8ZpzsfPp7Yi0E5hemMf0zjn09GcR79kDRMwzSUG03VJmwqBVWZzG/JE2wuoKFHIEw0iJTKAVcMwDSvOppdWlFZVLtSutefSvGEJxKIV8Xx7pfBbRHO9fwnSOSRqIJBSYEMRRW2hgenIetekayuWGetxBlfeS12IBlKNs3FynCRwqoPN/3IBMmy2F5J38/7P6bE0ZCGUDDKauweOWfV6eYr525ikrySKHJ9izshaNmXzYc+e9oa1KkIxi7aYSbvv+Zqw9p4ROcr+456daVoZL8HV27T+Ov/v2r9FodVHK9yCWzCPRuxpBth8R6pOls4hQNlifk9pqrsxkXe2YZsoKXWnFZ0X7Hz+UQIM67jdNtu1adlloub8tSH9TGA2NIma9MN0uQdTWC1SN4WoypsAk59uiMzqg0jn1Ak+dEl4ZQYigkzXh7zTCNuokm7ebGLzwbIze+GXsuu56pO/5HbKIo4Y2Yh3gueYUfls/jp1hFTc8cj8mJ7uoH+CiJwOqjXzBxL2Y8vLh+S99BqeeR+6sCOzJhNQdlEW0O0IUJZXqanuri63u0kkrzV87qWXYRITcyXiyhcAHL860U4VU0POMKC48ybSaayBTdD4UTkWRgC+dJFfHGVhCAIs6TbWlsUiJqUmPyaReI0EcKVJOM3GErS6CVUmc+fIVeOLmbSiN92KhXsb+LQcxPDIK5J7EYnlOWsFMfPK5rDYJwaN6dR7tSgUTe+LoyQ0hESfRnzO7fPYkgiRtskbsMT5jprRc9xyuoMMhrVhsjI/3Rsg50WvNvtaRHo6iry+P4dF+JEdz3McSGuc2iVLHmeJGHa6TuPrU88cWcfIwjb5NkysRMIvhZ66ArhEm4UJDL6bCMcQ6PHVN75ubnjRVM++y9cr/cdZXgoZKnwlW8tQzQUGfkUnFhYGCZQm1lN3maQYNnP+Gs/DzH9yP5WvaaOOkNg/XNv/LLEvYSLWKk9OL+OCXb0Y0bKGY60cYTSJfGkMrKCJSKCHd04c2a13SOpPmwct619x0A/XOI27dKlsjRTgw+1hPA1VZ6lFlY07ZLK1P7yzyGnOJNYvnzmo40X2JrNF2ekhNytMw728q6nok9RTwZULPnm3jidR8DTrz8QM02EboyWHNfd9GcLyCfW/5HNJBTJukFQnxeOUYtrSn8UR3AX/x0Q/gvR/7azx77wtIVFKYq82ikKd9hkVcooJ8L30212wn15csGm5Y3ghGVd83830/RTmv8+NaHYymBCwYjNQPTtKGkekigTDrQYvwH7OUlgHPExf483QmYG47MTGpxc9eMOs4WXW6WtvkbjquF26iawoiAv8MOCTvV7hAIq4WXZXDC+0Welf1Y9Ur+vHsXS8g1kgikgWG1w7hvv97BP3DGSy0NqO3VNQzpCwLhc15zby28sIcuvUqKrNNLB7LIZPqRyRISXybJ6icnzhS5wYA+JyqlbptaJU/VMCgxI+lpmq9OcDKwDtiGDzpjW5AlFQTWgku1FCDIaneqFT+ewd60bOsoPtLjCKR5eB+KCPz+myIykwV5dkqZidm0W0Q/DSZ1zgoHMishOyziAzCtZ516pLRRz9gBlujD+oEk3KFUU3ZA1I7jrPCGnInRx4IYyHWvXwEyVwCv7zxYYyuqiAar+nAUvD0znyO8joztYh3f+ZbiKX7rL4mFyKWQ7JnJbrJAuLZAiKZNBLpHCIJU9mQwoWE+LtC4Bk0/PS7AN6E9bo9wKqSgJnToXWvC/2mtDrWC3QZUmrtnVMCzR4GFxTvQAFLv6y/JFKDyDCWzrB48b1TkhL0ZwlVGxeYIA0F6ViTVlmUR9rYcNM/o7VuFfa/5qPItQKxk7qxCO6fexG7oxVsCWtYfebZ+Nev/TsGz16LrffsQWe6g1jKUGJDeS0rsGsw5zfOufaV+k0e1G1mX8uLtkeXP9eK8emw/7zkFfNFOdhuQe5Uz5GR3TjAHCs0CiPfn5tX4Iy8ZiuiKdoQvtExfSrD96BAnI3HiVi6BOiJI622Bnu7bTGomMqSUdWNtHHGprXIroxg29070C1nEUsZCj20oYSHf/Y0cv0ziGWO61kxmPb09iKbzmjRzM7OmIl1bRELs9PolNtYPFFEMtqLbpAAurzOtE5go23SGI6v46RiHFAiJ8S2pbFKIU+b42UdZ+uLt8aGyPVcQDqsDYiE7BU71h6d51lmtMIGFluLKPZmMDw2gFRfCsX+IlL5JHJFyr8YZhHpRNCqAfOTZSzMlrG4WAWn7VqLvG/UvzJ1RD6QWo3WKXQ/NOcLtdt4vXSld2L46VwG0STQP9aH1ecNqwW3/cnDmDo5gdzAIR1ZrMoFIjmwVevfWZ1UG8DXvns7Xji6oEDRDRNID64BkgVE4hlEklnJ10Sp501AjJkWNyuzJ1JGZcPqZsV5rQQAHWnII/PKfk9s+P1Q5G9q87imtk4hl+Kq1nNpkicJeLjeCn3H63UHsf7ON3cMXl9fGrvE+KMaIXQSI0JOUVedSznWWrOF9de8HvnPvxc7r/0ickendaM4QHXf9D4NGdzTnkY0XcQ3PvY1jJ03hjWXnoVaO4bdjxxApBJHrEVU2VQVuJGpjMHTdXhoSKemUn1GOIdYE5klt5arq1JbVBptTCjr9Zlqvnn8iEXlfl8b1IEjmgoSPbKNSr0mLi1V/0I29Li4iJYWcmhUjV/MhyCvXFdfM/DZAo8gQo2neErvX+8wXSaS3EKWCov0xmnX0bd2GGsuLCFsdfD4T/c4+46I5GKDWBK5lUls/uUWjK2bA2LzOvXUVuDMaqVGvwCEHTuhpLjI0qfeQKOyiJ/8cgv+ZNOfIuykEYTkc9sAQUvSvIZxcNNVax41tyF1lgE8pSnnw40u2mHcZkltOsurXri5Zke24L3RhtCpbkP6BNx860snE0dFHQrMcoRrqFybRyIXYmT1AMbWjaBvpBfJBIfFI8JiVK86HTLZhEgVzEAv9r0F+vAanK+xDioYxbbdaOD5hw8gbMZkU3L05GGkSy+awFMkoplkG4K3TIIBlfz4Q4eO4Hs334VnDtQZwsUviCRLyJQG0QwyOmkTGQ5+5MWkYk+XG5Y6VAK5JMrIAKmIgxgzFr4SueKntUeDF9ddGeYyabUdZGTlFiWPa388nw4w+UFsq+GMZaTC34EB4ipTv8lNZ3he8hIBwZ2EJlRudXEzbFgPNuyiGQ0RGy7i7Nv+Dfu+/n9I3/GkHlol0sEDs/txMt7Br7uzaIQB/v1jX0dvzxC6yS4GVpew4iXjiGRJK4sDrSjCJk8HXorxO1WzO41nMbJ8K2JphNF1FEXP7qJdZ5pm6gmcYZWSvJArO8m9eBdBllq1jaBMd/MG5mcW6djp2kldDUb3FovKNDrOJoW9Py4Cj4h2OObogBciz/Qt6ka6ohISACr055HuzyKVjyDIdNCttrBt8x5M7KtiqKdfgYenMp9LMhtDelkCd//sAZz9stC0puQcaCVEX28vjh4+gBgBNPka2wLn14kjB/GVb92iAY8zlq3HZedfiuH+lRrcCEO2sKz25yYNWKN1CM5YSs+U2tzzbCZW7cMo2WZ+3paoadK1x4zAYJ2KU3JBasdKrMCsX4mae0cIBVN3UAiLWQI5+WfTV2q362h36+hwTakHamm3viJsxcSRpH1KlHW4PSNtPjG5KDnEv0dRyPShHdBDKI1Sfxbl9hGE8UOmONKwA4G1NF//FJ7BPv4ifnTrA7h/60nbuNEUooksOpEU4mwPpfOIJXNANI0wFkUik9WwPliOsDxJmCg781kebrId4FbzksgOXwr2jb8mZORh9OBp5E9IRk6fTnLj+pTR+LvuPjjqmT74aRxlGfY6Rgk9hITeOoTWvE5PQdsCHtp127QUCIuFmE408erHbkJ11xFMfvBfEWu2cDLWxmOLRzCR6OD29oxO6He96R14xXmvRiKSQSxIKlK2Ig0E8QCZXFILvo0W4im7uUbnNObREmLOWiYamjGx5nEtbbHxPa/9w5TqlEoGvWH4JURaEzG8f2l0YvTR5YJzkx3qJSt51vuKJ+3IzUorHbXN0HzdeaGd5plGlhlXVhP1Kqd/aqhNLWBxsoGTB+YR6SaRjtLhjqbSRYFC2ggdo0SeaNBs+RDa4aJOr76eXm0C2Xa0OavcUrbACO8VGRKpFF7ctR1f/96v5AgnlROWPd0Qf/eZD2J2ahbxsB8B8ohHc4jHUgKXCPYws+CJKlAwZJukJblVugOIEqna0thewh0o5ytDcvOrEndX/GS3Gdg7d/RO8aQjhgxLTldahqwJiXSzlWQIPrEYvk6jabPOtAzxd1aWrG7diePsABdDn03RhFx29li7aKGnj1NfZFIxbW5henEPXagta5CAuRt6d84XGnSwxjJuu+cJ3HTvHgfwkdGXQDeSQDeaQoqbN0GQLiOnSyLNiVxRzz1wptogW44ySdpfUQ3fc237+WhlxIdWXxUKgiZClzAdYZ2gblLDn7AexJH+r++XuBpSJAueRg6V9pFRQIqTqVEqtiTqxdVgabbQSKncGfBSjbYwv3IAZ97wJQzGsnj+jR9HqtXGweos9qKMnYk6HqjNoBW20Zsfwpc/8LfIxPvRbXQQxqzWjCdipmFEBQ2nB9QmQZ99uyXhdvrmGhjEyOz1kj3t0IgWdhLwzzwBTe7HNHB5UhCgoP8rTzI1z9VfNAQwlkgtSalSgzmItJHJxhBJnZJtYaYh4I3AXtuE7DRZFdCexCRRO23LaAxEsTpI0rJqZ5mNZ4qqGZx06obIkPUTi+BE/UEgUlZfUPYligbmEGAC7yYxRBK7mFnsgycS2PnsNnzj+7+wWVG3mXLZND7/6b8wDnWtrs/FINBX6Ee7TiQ2jk4zC3SziEeLrn4n+GVtQipJiG0V5Wlrk00Bec8aZOHUi9W7PKlZtrCmlqE4gdEEHQrpR2TXw3tPwzdNn7khA6G8zpuIa4oTPv5w4X3jdVsZQvle8+ONJ4nSG1bBHrOCClNsAVdRAxejATKFJOa7m4GIlXnqtWbTSv1tHt0sWYzV1ZY964nFDj7wxesRTWTUOgqjaWWBNghFz6AC4pkehPEUYsksujECVQES6SwLGGV3IYOGRNJDeRglSP10bUNlity41uqhKJshhNLuWSS7x3pnVsSbgrpa356f6Taxd7iTlKk0h4xkoO+zfhEiSpZSzKlBOjE5L7XJfq5DqKvxDpqXno2+T1yLwtgwDvzBZ5CaqeBQewEHIzXcWz2KZ2ki1m2qyf937/scVvasAuIpuQcqlWIrIEqxO474uTYWWwhSUDDgbH6e+kskHKSM8K6Nau0MEUm0qU3DyPvWaqjemTl7gomxxY1q6cUD9G/OrZ3pFEESD2bF4m5mmUikhgusD9jsniLmE120wXFj5lg7xtBFD1Aw0MlqlKlVOqkNyZ+hoF09mEYjtUsqItq0Lr3nHDQXkhhITZqLdRFo8H3psMeTv30cP/zZwzrx/cZljfeRv3qLpchNow6yDUIsQwqP0k2i/lIMC3OLiHTSaNS4+eJIJ0tIxqkYGbfgGjJQMEAJ8zeBcmY8HGSQjxNJElaOkAyi1pSzDeH7MtUnF1rMKUer1byqgpzxvokb0ErVNpMJ2BsKTJDKSiRxoCUxy9vRQYp/56ZN2iy0PWumI3XMdx93oJGVh0K83bPjuuHPk7TBzUfLzocefwb/+qPfoRkhVZHrikMaZHExFYsDHOiPctMWkMwVIUVutk5V8yYcvZHkHQY1m7xiNsQ9qq4PD8MD46/TIL2QPjfGxmjDWoZEAd40W6RWH3qlC5EWPHFen8XYUUuULOcd4/Sil5QTtJmdsJw2uU5p46BqwDroIv6ZazD01jdKxXD6+tsxd9N9mOlWcaRTwewlq/D9Bx5U/s9ToTeSw3Xv/yKyhT6kYvbw+H0pChCdcywtcn6lcOhoY6rR2Cek4DVrFvXPDNP1LSwf4bSxGk1kc3kbR+w0zb2BKWCEFhxMobgZSOE0tQKbG7RJmWj8FDPNNqoRMrQAOKSeiCuFVbsmlUaHYmeOyCL+ruOu8nc1OkfyhZwBTAlSp7Bn/rRbqCdeRLxQA8u709li1BLmRXHThkw7WUe5z2ttszbu+tVvcMf9z4mkwV3Az7tixSjeee0b1DZJxpm+2eepafiE7x+XM4Iye55gDHydDmamZ6V8yB47NyxlhlpNysxkEA2LCNjUDSOIhkl02taPVXbTNuEBS51toF4sK2czyu9z2oqGb5wgUtargX/7GTHf3IwvFwNPcUmcUpeM7TeXjrOeFHU3ABKphDZHPJ0QOMn1zM9WDXejHhxUIObr83kR+SXzjVRbOtAvOvBTfOlYBB/7xGcx3RlGNdqLWCSp+6PWFdefDAWIHrP2TiCMJHTopLJ5taH47/9fW+8BZmlVZf3vG+vWrRw6QneTBQYVHRUJOuo3I8YZFUEx66goKDkjsYkCDTRIFgUEkSAqCGIYdRQwIIIISu5cXTndujl8z2/tc273//985YPdXXXr3vc97zk7rL322gwDS+nnlIsSKhGx3yMOoeh3ZPcPtGKfojFqIjTtxgeusFlT04LguRL57dqO4kYP5AAvtTg8TghIDTPSBymoi3ARYPTIDtJBwVpSyK81bPlvr7KRF161aqtmuf4he+HTJ1u5UbMtzYrlv/RWu+0nj9jf141Zg4OTSNs+O+1jX3r/J6yne9AbYJgTaoifR9DCrwFrjaaRqHGaTMCDzDjAJmTZrZnUG4MH5uDJqMlwRbV5B1WElAcBPH5WLkFIcLYXG0rN99JXinxpVz9wiw56CuPGmTDq9y370Gcvv7iaJOyhaFjZeC71YlZUGaUlfrPSSvVhdFgyW7J654uW6wYN9snyQmlbXG9d18uhFN0XD5xwMYHYW3vHrT+wJ558SYYvigS8ad/X2Pvfe4B6jCnfSRAAY5HBA3pzgZd4PNJSxMakwqJL2mgNYCwJ0S7q/rlu0H4R9MFWkgmbnJgUXpFJ9zGhzVL1y/y6HwAAIABJREFUTrN6v9YE701JLZPuslKZweCUtEgZyGNTojDiacm7iQoU/QlHcEWXUqmiFjkw4FoNdpLz7om4cE3ZbEJiABrfyhC9dCepprVyz1ijWVSFgByYlBCvifH0PNsrEDJ8taaNT8zYcSeebOmOfivl97FmGvZTlzSaLQmZBcOPYcrK8xLxNJkhjfgx15/rsFy+X/zubDavWdHqFmVSvUYf+H+JDasObkUScyXMXIkhL6CV2FDBI0YChbsL/3ISfkr0NuUxyoucNyqGh6Q6PTSGu+FRG8OeXAmwrWEsQY2mpT+wvy0657P2l7cdaZkdBm3VDafZ4x/5mnWUKjbS0bTmx/axzlyPffP6222qxJhtl4x5/35vs4P23d/6csstkcxLJZ7jK/qbRN0CgyvkuKJ9qvGBHMebsrlf5TzhcHGt3AeHFMMFwUI5OShqmO7HnNoIuPB9Ne8HNQiXbM1aMsiPKD8C/NAEc0Jy583y+xpwFQAsKSHEBmtNf4jAjfNjVW/X2ru6RI5wLJG0SmvW8ssnrZ4oW7az03JJJ+YrjggjWAmXNWmC6QREDu2pp8z6Kdn13/q2vfTqhDY4HVx8ffKwD9juuy4R8KYG+UxabKRCaOogQvN72jbHKUZTrF+sKDh32HnpGuoVBPoQiuf9eN8yRAmVV7ps6+iYLVm0g6YRZixv1WpDOTSH1yxjzToN9DQ05ARMcV+kN/CfAXZoXRTIKu1jmH6UCEO0E5r6FWJrzErWevsGLJFCsYW8c8ES+VetXJ2wzs4eJ8dkMzq8rXRWDRuUGDu7GRA+oAFt1VLdjjvhRJuaXWAcgaV6d7VCcrElWlnhR0KXpS4CoEk3G4AUDQ3h8JIDE3FIi5zSXpdl8p3WkevU/bglotRllti86/taUR6k3fcY8gANuQ6eJ+Y7ejSxKyjU5QTgBEE15/N6o7MeHlY9jF5EfS+WUvBwEgoK7CbqWQtLu23lPRfYlnt+YYVLvi9v0H3fBbb1+4/Y1I8esblF3db48GtULx0vVOzKm+9WEg903pdJ2wfecZAI7r3di9TMvFBJ2pLh5daX77bezn4RCogGsGztHAkgJBIHQqnB64aAQR42x3owhwSkNBDUnEIXROB8spzrbkUxNRk9dSo54uvyr2EMpNDnbfNxMWSy3FJGCLNz9L2QB+sgU7pxZJBpBXwWXoxQvNwat6W7t0RwTyMrCkDHbCQJAzipXymPAMG6NWsVhbEwmmRLBTA27ao119q6DUi9Wps/fvYZx1omSU6cFmod66tKRwJSLCMdpFecNBLeNxArFH1BtkFzStMJ3BjyOjWuBG0yRWgQIrX2TStXSpYipUh3WXdvh02MT1mxVFDDAqEu6U5P92Kq0daRzlujlrZmnTIVOXbKki244DCmcqEkaNZqJK1Uqemw8nwi4T+XT6nubNkZa6TGLJllVnLShocHbW521lMjvDaeMzDdxMuGmVUq2ab1I3be6gvlQYnkrrxmrX3jkttsrJjzHBcvrlZqB7UQKEDhJEFKB91L3VLqnpfHTeIMldfCwmKfIn2TEVKf2LDy3Tq4nps55ByZIO4cnT0lVYmga8ufPDCmA0TPKog+kCviQ3PAJgh3ydM5isyXI4d1a0EYqDatvHjYdvjZ+bbwlxdt9PMXWa1W8gHXHz/ABj/+YXvmE0dbaZ9lVn3rjtaRzgps+P0fn7Cf/vbvEkFLJ1J26H8ebDsOdlulVrHRqSn7ya+fCMqLQqiUO+XSHfaFD/67dXUusVymV/cFcum9sRwkV6NQqCpUzw2Qiv/UJhM+psS5o4B+7oFwTmxqDoka3mWQ3EJXar6JfVZRUSQIb3DwvAljIFG2MFA7lekUKOb5l/NiNa6TcIuylXJgKBQVG5sesVvvW2uXrDlLlEHCdcA3RRNBJsbfO+TNQmKhpTI/CO/mHl9pS6Nql152nY1PzIu8oKjIzL76pcNt0ZI+AS3VMmNMaPwvWk9Pv0Jf1irqZeu9Ei40KNlWoopAOIH0QH4psC/pAgc+LdGnUYisH0j0GPt8vlOMNxmFMP2PAxJbM2nw6EOZpMUYWGRo8cQcCed7K3SnqQMZWqYaVOr20AO/s6mpiu20bDdbvnilZTJdajKYmhux10JvzBeF1itqKpdCAwkH0eVk4bk3NMKlYV3qKOMMEIWZrV59qW0am1KE9G/veJt94pOHCYD7yhm3WLHZa0lEBQC1WhlLZ7g+b5CnPV4TDpizVKPu7g39hEmIxXFWUmlem2yPn01sXHVwK7a/uXV2TxDDYB3S0J4WgSQXqHY1x1gmwkT7wXfBK6G57nv0ED3E9AXhSwghsXu5bvbZf7eBr33YRn/6Oyt84zuWalat1KhaK52x6V0HbOdrzrKnDznW0oe90cqD3knhIFHTrrzxThtfQFKlZZ2plh313x+3cmneRka22s8f+7vVSGCouQUADkNy9Gc+ZP0D/SpBqLUrge4zfOOSUNcowQqIA7qraXoJDh3IZNpaVY/5+X42xxBqJ65kssiXcvhZP8JuR4Ep6WgtABViCCxEPkjdaJVcA8tbCYPUjvS4XNpFggPNhm3ZvMme/efzVmnVbLbARPWmGFYnnXGMLVm21IaGBnWdAvqkEBEGlyn4cjCwUa/I4HCASWXaoEerYasvuMLGJuYUVcgAJxK25pJvmCUrVipWrFIuquXP1RvrXquVfKQ/b0UW8V5DtSK+fyy7qQElGEepVgRsRfcYSl/CAEI0wH2o9Bb0uXU4SUPCVADQZxEUQq0YOVRE40HUWXOEzhFWoL570YVX2eZN04YIP4CVcI1Wy978pjfaRw55V1t0XDKv9arQZxBjUiL0onxNMCTegJJN422rNjszZxdfdoPqtRiQq9eusc7OjD366ON2y3e+bTa4r5XTSy2R7LSmDqU3FERD53xlBUHWEM8Aznc4i4jo06sF15oDzjVv3uk9LZgtCmEDDUBaSm01gqDIGObCbl/XBVSIobSTWNw7RQ6o8rSgNuBaVds2CWB183W72ZKLv2z1xXlbf8r11nr4cWuiHs7JBNxKJm2yp2W73LPGfn/lWut+80orUzMLnkSDnusNu3jtbVZRIGe21y7L7D/etp+V5mbs4f/9q03ME9pGzVqTNTv9a5+1VtMbDBQ5AAjkctJIjhxnvBQHUOUX1au91KB8jUhB+TxgCG16jvyyMVmfSLrHKLCJhJsjiwrpQU7ca9gCIeH/8vfQOkk47fvVDzC9uL5RWlarLNjzL75sv/7V0wq5sEllapbNlh1x5BH2uje8wRotn0b3///yFkG8d0rv44d32yRB1iGZaNk3zrrYpmeckM+9otB54XnHqwcVcKi/t8d7mBvetxrr/qrZB5X+uCElBk/Yx9wjPLV4uH5YolfTBIJQEhPfuwpiT4Tns4UiCBijvIijRDIHNWzX8Mqonu31bmicTsaQvG8I4zHMZ5xxkVUqAFYJNcNw+EGM/+tD77bXv34n6+vp13NCk8taSOs6FRUGkz6bZ0GRJtT3wQF434VCyZ57caM9/ue/2gc/+J/2tgPeaplswi688Ju2dWSzdaQ6rdq1yuazK6ya7vNGnGDoVM1JYLS9RIaFVfOKhOadtAPSzIZRmEz0tGW397dU2lGZxEO6qObHxtIhbHioHBdN7p3NEaQ6faO41i7lH9BILaAGbLUsn0haIVUXwpy1rI0N523n606x1I6DNvO3F+wfXzrfBsoJ6yDcTDlaizebt7LNZLO26q4z7YU//84qNc93/OFnFK7NzEzYP9aN2b0P/14PIJNs2pGfOcxymbr99ann7HdPQ1NzwEglK0valz9zqK1aOqAGb5DcwcEh3Tebzw9MnLVLmQrShiPpURfa4xsvX4kwobEbnrtiqWmfYwOCYMuC8qlhc8awLzZpyHNrTKWLmwnND03aMUWJ10bP6sYN6+znD/9eD1Oc2kbLyvWavf9D/2n/9q53tsPKWBVo52J054SculGc87qr5uY4SAcVMZlu2WmnXGAzHNwUYFXN9nnta+zzn/1ooDnWhAADRnHQi0VvZ9REwoWFNuIdUXBeV6b3NsizAA5JjzuE5tG4xDq5YyUOXqkc1nA5XJEnQsqFkwF0WrR4kXdKpTM2NzdrOcpDon0CInUoraEWy570mnenAKTTTrkwpC2OHWBkcQDHn3iEDQzkBGIymRGVDQxbjJTm52a0p1XHD/wDFxwEXUcDu2StTIdSld1228tq9YqcwAknnGLJRsu6u1E3SdlcJWkL2QFrDPyLNRLeiy0pJbfVIqwANMpwJiCw8HlEE+TB7ky0h0Zf85/AAG04P6KlEagSmpbyZBzrIxJGQD2jNZP8SMo3Pkajo9qyUqppKRQsyM2olQ50Wd+h/8c6Pv52a+Sy1nh+nf35xDXWu2HaOgiRMklJ1TToP1T9sGXVZMPG/nWJ1d/zWsnAuEay1495oFwrG4b2tkd++yd74rn1eigrhnvs0P/8d2tWq/ade/9HCvCx3xVA4F0HvtH23nUHW7FyRXuwFpZfPbsingfeqiyrh/o+jdDXKW5MdVKJk+tKDIpZAlPLJ+wBvhASbScuH9IQFp+NHME68jDE5eSJ4yC1MHlBZQc1MSRt8+aN9qN7HxaAwUEEZClWy/aGN7/JPvOFz7cxBO2D0Jboid82AKgyP2OVYqFN4eW6kbKZm5+y1eeusVIZTB5/nrKDDnqzvffgg5yjWy5Zd75L9++dVC0bGxsTe4swlwNIIwYGNWppd1ALRe0j2+GkmJD/ekNBRgeK94pfhPBKDXgeQWhBIX/CVEJiMBpjVYRIB9aXk/Pxslmxqij7eT856VTDyRnNhgQWzjvnCgdnE16S8464uq0+/1SrVGbV0IEoHNMPCaHFvZc6p0eXfG7/4IDNzxeUg09Nzcgrwo5Dfobcvb9vUPf76KOP2YMPPiIwFRwFeqeUK5Mm9tTXTz3Nnnl+zH7+u2etmuxRyZP7zFLfFo+acBlHiJF2aqpKhOyxrXt8UG42InyxHuetWWF2DhBjyMFizushoqOf8soa7NywCt4tlbfGULelX7eTdb/3QOveb2+rZxNWL8zbyJ+ets1X32d9r45Zg+6UVMsytTDs2qOENkd6pitplSMOtHKiYnXxNgHQOLx+XRC6YymHDpNLrvq2lZuEl2Zf/eInLNtYsO/e80uroiKhPl0ecMpWLem1zx7+YXV0KB8MaLKoiiGP8dw9KCuQW4mM79ROHz/p+Q7ibz7Eyr0qG9jZWA68ONjgTQmx3hdTCT+4/uVGMciqBE8QsYE445Ue2OnpMbvz9nusWfPaYZl5Qo2aLVu1wo478QTPo8OwMJDbOJ+Jkgj1ZeiD9QpNEOTyPlyK1/f09Nr4xIgf3FLTWkmogg372Mc+bG964x5+YDS20g/cyMiILVmyqL1+3HdsPyMHjjREMmuRIljj4DW3XwcOffTWREDkjJHKiPeNzkFSMmGWkFjeQWxO5TFAPRUBhNK01TKIIiCqCJgSaSNvxxx9ZqjJO0OKEg+G+vQzjrUEWEeSCAK1EPSrnRG3bcZuRc+X+49RhI82wYgmbL4wKwB02bKVVpgv2SWXfFPItvSypOjZtIVGRVHCRz7yETvgwP2UBnEQy7Wm/fXFMXv06Y326pY5a7Xy8rKNZMPBMHXree1ZSP6WPT6g+6UpQPUkTS5rqd0IF69NhwIFAARehTfBK6FG0D9opXzScsO9lt53b0vvu7P1vWE3a0JHROkBAGTrlI3+5Vl74eYf2cCWCUvXmpbBgoiUHtkgnuxHaZLYjTT5nl1t+rWDCr9J2Fl8wrLYi6m+23TW5/dIkydpN996p+2//wG2bLjPuvId9sivfmMvbZxTWx4sp0SyaR2plJ175jHKVfEO1PrQMJYqY8aBoFhjxkPIy6sjxkGVTJDWRLMpJ3kWz1lbLZeEAQkFuo/AHd7AvbUr9XMgvfHCQzXPD32wlw4j9cFORxwhDhB68/1KdcFSiQ77/f8+Zk8/8fcAfDWsSG0y32GXXHZpmDcTR4iGubNBwRLomzzXieh1q5aKYqoRTUDIGBndYFeuudWKiLgHIbavHvkZ6+/zaQYeaTCipNump6Y0FnN8fMyFC8JYFU+pXF1C9yvlCTfGiA9EA+b32Gld+bzNzsy6sEGpqCYPfhaNIx5GgntCrr27yc27A1QKH5NoeJUsq95hNrP/DmGlS/Y2rb9/wDZvHbXV513Vlqd1XnvWVq1Ybp/93OHaG5AcYrmLkBnecFWySt5LrnUI/bdxSh+lrpjrM2iMa5iZXrDrvnWzJZNZGUX6zXlNVbX3nJ122slq+O/tdVGFqenxtjh6odK0YqVp9/3qeXt+S9GmFlrWQjkDZU6xv+qWGNnjgy1CMMJJVIYWmg1LQ+1LmJV6MpZfscRSb9jd8rvvaLmVSyw52G/Jzow1QOUysEV8kjj/y82WbeOTz9qGX/zWEk9vsNx0yTLFqjXSZpk6OXQ9dAGR7AddWno7s3SZBMoknpuSSm/Wip95k82kK9JdwjPyoFm8uQLMGTaBWXffgA6Kt5Wh0le0cpWQrttKxYL9+S9/sz8/s6mtbkC4lkulbPU5xznNkFJFBklOZzl10zNbZtSHz3SN+SchICEX5Q/Kz4R3YgIVGG7sWldcKCwf6S2HDhYMDRzwKFmjRosgi+LSrp6zcCgoNThzykN195z00GZF0MhSOrOUbR0Zsx/cfo8sOb9XrbZsslywK69eK/pjDOXFtQ3IcIUh0uWSIgcpKyh3Z/zGgkLCeq1iU9NjdsXl31EDg2eZSTv55CMtnXZ1TAAfNQJIZM37ZQuFBa3bkkWLdI08lwLicFLmN+Xh8sahCYBDENVBkEzlIGfDNEKEyksLBT1jhrSNEoYDOIn5tU0TTOURFDxqNevt65PHJiVD4havqq7aIDKPfI5SmUbTXl6/3m6+8S4dZmq3KgV2dNiH/+sDtudeu8i4w8FWGsOYmS5C4cmQLjniLYMRokz2zczsjOfBoU2UfURU9sjDv7G/Pvl3HUxNWgy6VGTNr33d3nbwe95l9TrGpsN2WL7cJiemvZEeIK9WtGwiq8aCucKs1ROdNjLWtJ//+Vl7ZbRu89Zjicm7H2hl+rots+OwZXbocxK0OvcJo5qWZLQDOlOlqhUnZqw4PmGFZ1+16rqtNr9ui1Vf2GT5essyADpYA3GAE+qrTVVduUI8ZCB1SbHAYnIKV8yXQQHdUnqiPtOTsspn32YLncyLQYXR66hsHhXwo8wLaHjKNWdzHZ3KK5B5RWVidOuIVYolW795iz34iydDkd+nHCQaLfvmxWfoUPK7CwvzwSPkdIidoOJhr8TQOVzBa3Ko0VjicIjHvb3MrIZGeV0T1DSyn7hXCbABPqElHco11DhjmByBKZHVU7mgtJgXM4rrUSN6kvpx1qbGp+zG625p85OrlYZNFgt23U3Xa21iGCe5sEACATBsVEGSg/QJoTlaX+UFKxYWlMNNz4zZVVfe5m12ut+UnXHmcd4QENacziLWgC8iFbwjBg0pHQ4sX52dNEl4VEHLJlEN3pZD4ioZfvDcM7fkwbhvgUWZtA42/8ZYi0KriY7uob1P12ca43HRv8bgOSHfQVS6wHg23jCDyob3mj/x1JN2//2/CGqWPpWQ8P70U08ytlK9XtHBJWTnQzNpIqKsTU5NKoUSSxA0GK/ZRe5e9AaRQOGN0xtY/8suuVa8AOZE8QBJigTCZdJ23PFfs3QGz+nenCiCz5EKB6owRHFBuB5RORDnUrloOaLBWkrhf2Ju3dOtRKFszfmyFbaO2PzzG2z2n+utsnGTNcamLQ90XvN2JuW8tGSFso/mnQSqIIOs1QGDtwn0t9gGFSelCUmNyhPqg3RVBcKiTpC1tNnL6ZrdWt9k//3lj1oyBz+1oBwml3cAJDJusGoKM7p7dCDiYGEeNCijxHGaTXv2uX/YAw//2SoisGdU68tlknbc146wFSuWtjVx2QnaJELWyUfTVizhdX0mTSQ16MDCOop6VMGbxFolHgwAAtlOVSbaA5uh3/nnx+kKeE8JxakU41PpIRiwebhXjd4gfWm1rI+pgPB+az6i8/qrr7VEM2nZdE6o6VRx3q656QZvRQylJZL9tnEMqDYHq1YpSeGhiQepl2xiYtx6u/M2OrbVrrry1qDVxBpk7JjjviSkXrV9zQRyCiiHj9p2rL2io8XGXLJkiU1MTbjxDqJt5K2E0vLAGimSF/WP+wYU09CtZErfx3vG0lKt7lMN+Wx6a9nc1Mw70WzSHF6vZPjfnf/b3d3lhieTViSmAW8yFFn74X0/tl//+n8dmMphBLxF89zVJ2ssCXk841kgzfC7maR3xnnpzjW2eXZ9vd02NTWlZ0sEpucnkgwRUNNefHGD3X3Xj+VICO9pKPAGiabtuc9u9vGPHyrwy1NPP08Ab3FWcmSjOcbhyqS+5kgCe5SSeG6PtwsKVfse6ozUEUVXdM8oUCGIyIlYEb6ilKWHZZENtY18gcV2fSHPdfiSWnxoKxOoxWGSQkHT5rIp+21y2h7LVNV1ctzXP23lwoxyP5DCyelpdYSwwdkkbHDQxu31o8i5uCnQTz5306ZNCqXuue9X9uK6rQpRIXV3pBP2mcMPsX/919fJikt8K1Abe7p7tOHkeekU1fDk7YTBlB46M0oWMqhO8Dr/ooxCCcOHNbdVNxDOzuVUQBe3JzBj4uKomSMYxO4er5UK4Q80SgwDh1bheXHB7rj1eza6ecxy2bzyp9ly0a6++QYrl/zBik4phNytOmR4WX7CZO6rUra56Rkb6u+2mekJEU82btxs1157m8+HSpjE3b961OfE12G9o4ER2URytH6v8kKI/pUrAvyQ5CFHdxpnwuhKwqty3RxSIeSphO200yob2bpVLLA4VMw1rb03Soqhkjjy0ZzbaKo+xlPU1bBm8IsLCz5cnIHogHA77rijQl0OELjNjTfcbM8++091FZGeYYzz+R47+9wT5Ol0LyIh4bmzNjc14cZCpT0veymCiXTe0LvuP3fmE3nyfff81Na9ujk0X8AdcGNKmnH8ScdIXkh2MJwnnlds1pCoXWjMiHs7dq1JXIEvDu7fd3l7S1aFsC/U9IDO1U8r+UpnSMnbhhm4PhOU/CUucuhOidKRQdlBnxFqwRqiFUTW+D7vV0iYbUxV7c82axtyLWuB8taqNl8u25v22MkOfPt+uiHCRQgQ3CAT75jAjuedmpy0TsoMCcJaNk2XvFFvLzKkjNPskKLjn578h11z/d0CJeh3xOO+86C32CGH/Jdeo4bqQCBwEAjrTtO3o67Sygo1bl8PBxpUXwxsp8ikicin5sCGecB8hq83qDRtW2HMYmjUj6FtDGtl4cXEIkzyMN1HZjiSzAb+1c9+YX/+wxPSLyY8nq+V7AtfPcL23nufYFSo/XmPq64tWHYRSAANaxWrV2rWrKF1PKcG/C1bR+3SS66VvCpe/i1v2c8Ofu/bVbNeWCjKiGZTaZuemRGxnnv0JndXT6SWyWu6uvOKFiIqTq6D2J4a+ANnm9fxO/wuh0jN6LxPB7N4UbtwkbyYctAJDnjFmvhasx5+cJU/57tEOxSpRs7AmzHUxighw7RdftkVMk6u1AEWkbRlS3ewI7/+Oe0Xyb2GUidhf7JJia7Te8nTSf3J/YpNTg7c0+1lsXAu8p3dViov2FVrblTLIt6fL5whTm+XXXaxQw77EPRkPQNO1PaOh3uSgQ57UVUGxoeKiaeub/f+mOAnV+wvBQyNDNmuTqlDGw5mRNO0ELh39ROzeg7wYVFSWB+K62yMhtecKImQm/Lgs8m0zTYqVutIWWrVYivsucieWZixB37/uKwPYIFarMIcWcCco796uA4PIbl3eqRs6bJlsv6O/BGqzCssZTMPLxpqgyIgeXScIEX6ysYNdu7qa62JymDSB2qtXLXcTj7xCOtI5iybY+yDK1q4z0zooWB1NOM1rIUsv8Izn1zo9V1XamANfZN5eAXgw0NwZNkR8RgWubfmMHmOGz1tO3pRLdhJJuoECaqP4q4GttfLL71sd91xr6WYUl5vWalet30POtA+efgn2yUUNTyEkp6Xspz9QxkOnrLVncIIQLJ164jNTM/bNWtv8vJW0+wrR33ZBob6LUekEuIJs5r6pNUvqwPheeXM7JyQ20gsiQO4AXySrIU2IdEAtVWXtVUzvlKUvA5ftiNjC0Fz2mv52wZno52t5pagEaWy5XaypdK7Ar+AaqoSl6tYoMpJOMuzuvTSK2xkZNQVP+T10/aW/d5oH/3oh937yXt75KNUp4bCSF4RF3I/7DkcCRRNwtply5bbxo2uQ6W5SY2Kbdo4bnffdb91dOa1z7jGBdDyjk779KcOs/7hPpdI6uiwhdkZvYb1Y9+7MD8sDJ/J7KIPoSQLkh0ObfvgeumD2l0gGQQ5mfbBDQQAWQNCXWlMIS3kaLQCZaRbRHxvWj3RsGZ3hw5poydrXTsu1t+ruy62Yp4e06QtTM9ZpVy323/8U1kVeMOIVZMPiNFUqdgXP3+IDfR2WblGWJyQFacPE4V58kg2zfTMhKw23+/M5W10dLQ9e2bz5k120IFvs5nCjJ1x5hqbmCyo3MB9dHXn7MLVp1pvvkfavpoWD8ocvK3fO0iqN1XH/IwHyn+RqhgPrkJdqX94Ez3kBCeLeHPCtoPrDClZ0TAwTQIFgeIWYiEPP4M4t09m93wsHtz5uQW77JI1AlDUcNBoWe+yxXbGmWfrWtVmp3JJLEU5G00IbzphCzNTVizMyIsNDw9pzX7/u8ftlpvv1OGrNZt27upzLNvhhzaWSBhDRxrQle+yufnZdhrEYY8jVLlGNjyhJZUEvDkGItFsiNwwPT2jZ0Zk5GQJb6cEwALRlv5ZKMl5bTuMlgxhMT+L6UA0hrl8t68nayREPtS5ywBOXgM+66zzbG6WecKu48R6nHTy8bbNwWmqAAAgAElEQVTHbjvb2PiYT2+kbioEuGEtkPhwPaXinMpy3NPs9JRyV6538+bNiuqUE2dS9u2bb7NyyaRdRaQoDKBRs4HBAfvCFz6pzq/ubk+FIndcVYWg8SZCShFcB/qnt4xGFpw0wMKA7sSTK/d35hT/C7pRgme2G5YVaV78EuPsherKEzSsmEtasi9vM4MZm+1MWKMvZ4munKV7UCQEmnc3T7jXSieso5W0JkwUelvmS/abR/9s6zZPhPpgr1WqrrqByv5++/2LHfDmfUUOTwf4HlTW5VOj+FjgkKYResuKuQNwwGKA6BFi1Vslu/CSG+yFFzaKLcRCQB6/5MLTESG0RDpq/3rYFVMBGRKQbMm8OpLpBBXnJgtICdPzZP2V6/ng6HSH82SVF0ZBdhD3KNcjHV5y3RD+BtJ6BCZ8j9Jp40oeYglJRdEbJiDqX/7NK9XBIpwgkTJY2ZddtbZdP465UvTokigNk80b1bL0lCdGt9pAf78Oyy9+8Su7796HZEQofFxw4WobHO63uXkH3Pj9DjWsu+ffOjqqTQuvl3VgPRjclksnbX7ePTAhfnFuzhqAKxna4jyEZeojXkXjV6gpKyUCw/DSGOuIlxUoKgka9lAct+kgl7P5/J6kl0bomWH2jk9713NGUUTPqmDnnH2+Vcre9+yAUtouu/xiGRfRDquw8ZjMkFMoXFVJ0D17MuGcZb4Qkfd+aq+5x9IXf7/xhu9IUL6js1v7gSiO/fXJT33ChgZICXx+kaobNKyEFEZaz6HfV6qkgVYcS4UukO8OUljNn1btTzFGVrWaBJpPqkgvACKMOaynTPKoGbxfZ8LSOw5bZcWAVXqYMNC0Enlp0JnFIuFBgemxQjQnk89I+yfwnRU+ohvVqNvk5JT95IHfWJ2ByTnGUThyCsCUyrTsy/99uAAgWtpU9gHgSbvYF1azo8NHHPKzwWFU+BMmnWg2BS1lTXpgG/bkX5+ya2+8y8OrdEpDmc5ffaZlMjWf7RsOXDLrVEIeOkwlQvToIWUs2sOsIdlT6vASyPZfHiIH30mdMhA2hH6HAeGANF0AY9IiJszzsJqNKHazcno2Laiq52SIrZFSeD9x07598y326qsbVQeVbEAyYZdec3V7M/D4I5LP1cQcmmiJjQzIt3nDK1ZamNdY0J8++HP76UO/0rNHB+rKtWsFVM7Ozckjo1jB78SRK+R3ceNFD0hqUi/7QVe/q5kMqBpCirOiHgqdpuUTAQMqDYp2+Dc9q573aW5wkGfNh1nBUs9QJxGlFUgyPgiN92Y/aDhYGPzm+sxuhAnrp6dn7dxzz3ckmoMIut+RtYsuOl9MOxpNpECCXnMBbe2MJH6IxNi/1JcVNaEXXXO6LV/sryg88be//dN+8chvJHkjrx+ihaHBXvvoYR+wTqIXqZsglMeM3EhqaVl3l3tz4R3pjMJm1fzDJM34HCNnPvHHnd7cwtPy0DPNhC1Y3aqZhFUHOq1/r50ttWzQios6bKZZM+vqsJRKCPhLn/ZO6xGAUnFmTjfCDBUAGG6SBwBXlUXhQuK0MR2erIeCExMT9rv/fcKm50loIIZ3akwI1rhaL9tZZxxv1qhYoeggCP8pf8h3yqry/s4VLdvKVTvpYKmpXZPbQCPr0oJCauTo486S5ebmUfM/7ZTjbcnifpVFWEwsp5DYdNqe/+fztu8b/lVhqELHunNWI7I+PTOt2T+AYpE2mZVkTigBCb111g6GUGUwjXRxcEHzlkLfJz+LpAQeFrVr79bi4MY8mfAOPSQUIFnPhP3pj3+xe+75odg+tIpRq117443tvBlvHRk98br0WVnXqtq8ZbO8R193p8Cq226/yx7/w5P6/XRnxk465RRFMOwN6qHkwXEEJmvERoNGOTMza3vusYfPBgboq1VEzKDEQTPDYL+TZGCW8ewJOVkqjBesN6K7GBoDAsE+Ep4SZtDyORFoEodZHGSK+97dJcE5rpnwVwbXx5FieNl35KCFhaKdfsZZDsIS6WQyttPOq+yYY76mKIz8ER0pDNj4OBEg+6aivcs9VUpFb2EEoKOVr1jUGm4fyn/rmpusXKyLp43KhWZEJZP20UM+YCtXLRWSrxwWOR3uLxBvyHdhyEUBOtdjdsCP/aIDLCDO8ReF0D//xCEtDqmhDtiXs3R3p7WyKUH7XT3dWox0i1EIiGjCrmqoN1HaRaG/dH52ToyoqExIo7dCmHTa8l3dbe+NvjEbnwslb9V8n0TCRrZM2e9+/5RALjGOArm8VK7Y2w58k711v9fpYLF5RLKoVq2/H7JI2nKdPfJaGJHFixZ7eNZqKnf76xN/sl123lldSRzcY084x8pIodJHm8nY+973H/aB9x3c9m4sipBO6o5SE3QtJaGjgafsltZDajYbQnGxtxS0efsDIotMbTvwmmWwwgQ1IdUB3o80Ov1uQPCrNe+KifmNpD3xEhm0f/PWnc/bhvWbhZSqFlqpaDzIFdddGxQPGS7shiSGlfF6+O7gwKA8VKVcsPmZadu4Yb3dccf3VYME61i0dLGdedaZAlbmCgVDXoaNxf3iDWP0gAfmGivhcPmwNUf0ObxEFYipwWQDvOEZahpElDYys6WLh0SiIMWhTMSG17jJYPw9WnMRPkJuIiRI/YpaNMDc95rTTltieLH5yUHZXzxH+mVPPe0M77flNR05e8c7/s0+8MH3e5seTQjzc0oFXC8Mj1uRMdLhpSxYKstg4JW5Z54/pSUiBwz5zTd9zzoynS5HKxS8rNz2S1883OqNsgw468PaCMRUq6x7Zp4vh5k1rtBRFSYVOlaRUmqnUme4hsTdV50gVDnmWq6P7GR6nwgeWDRhrqjC0DBqMlLAiO2xevwZ65E6BNKHNRsaGvJJbqGJXu6e0LzKFPaWHvAjj/zOKlXCVAJF16SqVetCHo86+tPWCrNyya+XLFtm1RrT2wGuvM7a09trvb0Dbs3xbI2GPfDAA/aOtx1oiRY6S027/Kqr7U9/edYyGebpJuwtb36TffmI/3a1ytD8r4I5qJ7a9OLwMsZpOgMGSwuQoCl1msCHd2H+q5MouG4HojwfkuVvxfIPyGWwoGrf2zbdnVBRHTTybhkh4gJhNNoyFMI1tCorgkAuD/GkaeecdV7IP/01qy+71PqHBkNrpQOlMe/2afF1MaW4xl133VVtkYBGk6Njdvmaq2z9xhFFJa/Za0/74hFf8p7QdFoHi+aBXKeP3fBD5uioDkJob4zElMgG0kFGqI/QmQYOt2xG+BtLTGAlDgjVrYqGV5D4ZSN3d3XJ6GYyQe5Xapo+j2lsfNzXDGYZ1Cf1EGMQzdcII0FzQb5bA9fOOWe1vJy8cCppRx51pDrEmF5I9MM1k8viff05IgnQtMIsA+U6bWZmRocMCdresM+Q16GL6re/edQe/+MTCnmlJ8UggEbNPv3pw2zvvXe16WmQeL4f21aJHreN/4yht3L60EEmkC6kEBhOTZlkgDhVi/uuObkVw1qFs6F1T4AMlEAU9rarAUoJPygS8HssUHTnvG5qckoW0KmECzYwNKRifDzQcVwjUphefmlpmNWr6zbbU0+jLuiWqMyhltSF2XEnfjGoaTi6uXjJUt00KoPk1gIzmi3r6xvUweUQR34s+QjhWrVcst/+/jH7zq3f10hHCuWrVq2y8847r93gz/06Z5q65YKsMNQ28qVysabQT8oP9Zo2sTYh4Av86HLRXnrhBVuxYoUsJyGfT1v3QrsAIrE6nSmjNY1lJrxPoiUghTxLXGV5fS/bOLnDSzTpVDYwqqB55u3Ms86xwpzLw/J12nnn2bIdd0Beyz9bAE4YKRkIIXgtrpEQdGCwVyDMb375P/bjHz9gY5N0ppj9x3vebfsfdID1glXMzwvlx7suX77UXn31lYAB4G3CoLVQ22ctZLBoZaPHN5SveM+a6Kt1l5RVe1/Nli6lvFfQurPmZSbC5xgxilF34CmrAV0enemrCXhZsE7V2hvyiqD/aooP9whyK+yDWbSJpD366B/s7nt+qGgBh0LIf+FFF3o6orDa07CFwoznrgCkC3xG1hbmZ6xRcafE/TJOBoWVQamNgOmYXXftjUL2yaupS6tslO2wo4/9iiRtOSORLgu7bHx8XPtGHPcAlnluD+rskR4YgqRZG6RSOT0v31tpS/zoutP0xHWKQ7VOmyBMPI8oq48/SFilVG43F7NIGkhNrYr2JkTWVOf0dii+D9sp6i3zQDSqEgHrvC+oUFRr2dxC1X7y40esWk04Yi3yPCFVy17/hl3tfe87WA9d6KqEV6HI9Vg6l9UNUg4CyYtJPIsDQV2zS8slhV8s1rHHneyT0TNJhTHXXHOdX0NonueAsHj851I7XjZotpLKQ0UwVygPcJBRzy8US01xD/kQy6cWuJCLcX/R+6YgNwSryibyzQkguC3MjkCPb0Lvc63VaMfjetzjduTz4rR+85uX2+io0+94/eeOOMLecsD+Mn7xMPtu3/ZvnmE8uJVq0cZHtqgDa82Va21yqiCvdPSxR1tPX6/kQjl8REwYLs05azo7jY3mU/x8OgCRi9ZfIuRueGK4qrpk3YXLBZIlUzrAgGQ8b9YYY4j353mR/ij6C/OdQKNBnXm9lESCogp1eQ4uho9n7FGiYyUut+vo8f0//In94pe/DtMinGNww403WKm4IGE9ACmuNYoDaO01+QJJ26rVSs5LJoxm5pK8ovp6MTglu/ZbN1pWoXnQA6vV7BOfPFy5LXVfnS9IS7wnTADx1h3gigYpEjA8vHf6J9zmeLAdJA2i6D/81knbBNFbXjNTzlKtiazvVoa6GjWlpC3Mz7fRZiycgw5Nq4fWJiXRKbR0nUYoRJnp9Wj+hG4QaQdlUQsoaaI7N481ee655+yfL4xatZ7UhqEvMiJrR5/wFRXHKahTKlWfpoj+PCSGNBesu7dHh8sHOIdZP5aw/r4+bRYOwKc++XmrI8Kd8qL5TTfdFBbc5wBB/YtKA3h9X1lQR5hAgdlS9fxTOUk6pfyGdYNcHz2OvEoYiAaY52UD6rEgvY4WIs7m5Y5Y4nEv497ZzSgally3jEmt5DlzKmX9fUOSaHnqqafse7ffpWfDfwe881126KcO176OdNNISfWb8UNMGAioRJfQxNiIjW3dYt/97l02O1dUnffiSy9VZ4/wCKaz5/PKAbu62JxJ/RvyC+5ZXOq+PkVnkDMkSBBCZ1B5rrcQFDK4K6UjQbxBjQW0iBKtTU2FpoqEDQ0O2uT4RDst6+/vtSnVT71dDwNOvk00ghGgzZBGh8hdJtyV5yIlq1TtqquusY1btjgwxXiXzk67+OKL5QyY1xv7XKVlVnP6Y2fe97eoljVaKoOkU0itYh5//w9/ZOvXb3ZkO6DW+a6sfemLX7Levm7tEcn9CE12MM0bKraNo+G5eoupH9QIAkr5cTuGYvx54t6rT1So7EOjfAHFvcz5MGtHvJj76pYB3Vt+zmHmAfBhqqSQPwmZTSuUxDrr9UFMjAWkQO+slIoOC2WGnm7mzXpozWu+e+u9VqxQLvIcG5Qaa330cUdaR44aoHsyPodwiNwTj0sNjIkEg4OUn6DN+dgJXouxIc/m67zzLrBn//GKroND/oMf/EDXIoApCJe7JU0qf5a1C6oDHFxnS7EYgSBOe5tANi8NcB9x3WL+F8svbsx8IoTYVCHfUXmMhxoeGmkKX3pg8pQujIekajy4IMmICuB9Vp9LyOcHvX/xMvvG+ef67wcOefTwsV4vDrCZjY2N6v0mx7aIVLB27Y1Wrbm863nnn2/1pkcVsSdWWEgKI0uI1yHWFsZbpUTyQ6YFhFDYm098IBpeyimOHp6LeBGUMMnbMAYYAg4/h1czk8MIEQ938eaO+rqQvKOrGhpGDbhSUV1YDKka2ljz4qjznnGvnHLy6TZD6EnbZSplb/zXN9rhHz9cCPb8grdoclgKc3PtqQmkPzwbPc+sWq30rJUDlwDQEAJs2IUXXaLuNEeJHbR898H/x/bYYw/dWxh0IgfmIvnOVch1ODqtMlgoHUXHyWeKeRV42yoTxUkW4AA/vv40HVwv1nuNy7WCUGrfNjdIag4wi/CaGmhNw3E1CHr7DF2Va5Ipm5mb1aLNzc956EKY1dfbbufiQM3OM8LBgSRR/SgJ1Gr26ONP2LoNE1YLTfuiM5rZ/ge91d75rrcp+S9XFrRZevv6pWkVwwfCiojETk5O2tDQsCiOcDCx+Ljq559/xdZec5OzojJpO/PMM+0t+71V5QG1DYa8kzXx8ZGOMjt44iwf3q9dZhHAFLS6aPRG/IyJ8YwuDeTzapm82FvL0uHgAn6p40gHFAzUmzH0uRTbA9E/Ug3lNYPkKb9TZJJ809Uy2ZTcj9Q3Mx122dVX/X/qqzwvv+4QliXJp3P2wgsvyivNTI/bKy+9YNde+23xfTvyHXbOOeeoIcKHbfuoTJ4/B5c/RdmbR6DAPB1ijnC1IoMtFDuUv8AHCGWjvE3M310s1nNwiBaRaIBnivxdZiupdVIhposbaFIC/HKh0i6orxnFjYbKiKw/xgQnETuv4CMce+wJqihoHEjC7Jijj7HXv/71Mi5TM5MiXajxo8kAbHdUHNyobKIeayKnYtkG+7q0z0g5Nm3YaDffdIt15XtEBfY6f8OOO/5oH5fZpPfcjS+/42lZMHA5Fw2IXnR7YEoOY7upltsaDvyeEw/edLom0vNUeWgcRh5SpeYgFDdBmMvq4WFBxxYtWuzspECtw1I6WuZeyEsk3iBeXPDal8acNCBtw/0sW6HoPGIvMZS0gbjQdes22q9+80erUKZrJKxKY4JCtqyddfbp4tmqnzPwgBl1QdM1G4LWv4hww+jRjfO5INQoBtYrNj251c48a41VkNbs6LB3vvOd9uUvf8XQ5/Vaczg8gWYXrSHXuD3yF/NgSjryyGqccEK7AJVAT8N7VGtlARNqzIfJJaCFHCq0SsqaekikyQZi67hahg+q8rAX/EejOgFkJsfFn8XSX3zJFTY5MacOFkpGV1x7jVNRG4HrGmYUsWEIDZkRBELK88Iw8iypp6+5/Ep91g477GBHHXWUJGzdw2+n0ZzyziYMrufeNevr7bPxsTGV2DD6TlsMwFU6LU/IYRG4Qm0fWVUiGiKikJrJE0lTmbZMP+jkgLCylENnsoqaRke3yijy3FnnOC4Go8rokZg/I2DOvlAE0NVjR3/tWCvXvO2U91t9weq24By1e4wCXABq3KJqUnopLrSbIsQ6C5GKxuWEkPu2m79rr7zySpjc58+PMtOb3vpmr90DPtW3lfboN+ZecSzsUV5DM76GnGsfeVeUkzRcjCDiIE4KImopWuL+605qyVITIlc4wB5+IE7FQxMTRU3AziJxJoeLo8F44cN5KpAG+IBY4lHZgf7SojcnYzUV3nZ1e100gF8R/QVM8k00bb/89eM2OVmU/AudFa47lLCvf/2rQoMXL17i0wPZiEHrSXlXl4NTkZjNdYs5E8oWE+OjlmiV7fgTzrPZYkWh3YqVK+3yy9dYPhgO0Go+j+ti80Rks81cCSFLLF+ogyhI18a/c4oBkCJ3mZqsE8QJieGvIHRmVik6F9WNg3teR/C15GFwtkdBrpTh4SEHpjA5ZoXCjOqkd/3gR/bM35730Y8dWVtz7dWqxQauR2CseY0TA7l5yyZdmyRiBC6lbMvIiJ1z9rm6nje/6c32mc99Wt6Wnmc2itrN1CEWdLe0zgyy8kFvhbl5eV5+Z5aQlAMS5hypw6bsbCOMuLxlC0ZVT7uvNYJlvb39CpkRoQMzYM9QNqJ8hJGP4evGTRt1L+wnNbS0kK/13LFWQ9cpTuZzreKTTjpNooJcE597+RWXK0KQqkqomqhvJmA1Cl0hFgklJyWpKIoU040DVfcG+gvPv7Dd8+zD3lp21tlnW61eUkO/UPXgiSXXm9vGw+bCnJddUelRxqMEv6Gse4vpHPfP+/I92HqS8OXgikwgAGTbgOGFEghdWtaNeqF7gzC+IsD09FjyPW6I8gcfIP1gkcC9JQtJDh2AVktkdulM0UDd06XEH2OANSNfZWP193XZ1ol5+973fmKNZlKhK3U8NvPb/+1Ae+97D1Z+Se6LkvzwomF5D8Lazi7E3wBSumTxBdhElhIGoNaw8bF1du21t9vLG0cEbpEL3XHn92V82FyQDWKtDKOkDp3Q3xqNAmsRv+dKBXHiA43mDsqR15Jrce+cVh/9gZcFkeTjIBP4a7f/UggehMBleDRMzZUXiDrY9KxHvUg7Hn20DXvyL0/Zzx76jU8jTCbsyuuu0WhG16JzBQ82iCis1rLR0RF1WLGpyDG5TzbELbd8x1566WV52z332sNJFqE7is+ltkzTARsIYFEU1nCARfsLJSnm6cxMz6jDSnsmIs0IDII0Q/VUzXSb8kXctF5OyQqrcKTXpWR4koThfM+F45taX4BBPCvOQWmR69/rWlj70dExYzby6aef5dzwTEYp2iWXXqIDzz1KDxt1RdRJAoCqSCPhz1CrGDANX1GR/Oyf//yn3XH7nQFdb4gAc9BBB9p73vs+9TsQusOum5mdFEMs18mUQq84COOobxsMxxwnDBtGZXZuWpEb9yiFytDMT5sga4G4ROK+a7/egg/LFHHGR5JtoVAfmRxYd+QwY60MaJsF5IHHflz1m2qaHdaxYLWq53wc/GLVxc548EPDfSqao+bAgsVNUw6EAKkVZDI2OTlmjzz0R5ukKRwVgjINED4I6tRTT7RMh3t9lpB8EkOhnKNMWO9KGfkcxsQROlngUFeemZqwf/zjH3b7nQ/pCWNxb7zlZlk8MYkq9PXStVIVuX94eJErFtJ+RoknoIYxD8UgicqoRnifL0w/L8DN+vXrbeXKVQrTOejRIkdiS7nITFW/Rr54QP+vr1hHJ4SOh4nWwnq1ZPNTkzY9O21rr7pRJTJSiHPOP88Glixus4TwjKqpJh0sRI2QL+RKSQ8Iy7xs41QPDvj8/KyuDSOxZcsWb1ur1cMECBo9OmxuZla5JPeve04mnSSQg7nkHjWi5uSbEYQkdfGKgHsvohzWGw+4aHhYQgaEuqC4eN9tRtIUzipCCaCh6K40uLfQiMrLGUgFZWbWZqenlbsiLnDp5Vdp/TE2O6xcYcccf4wNiIo532a+8XzVNBIQfcpSNIggqgciiYpHviNnKIqyRtdde63WRg30zLhNJ2z1Bed7ZCVpHs9rOzOpNiLeaFRUfyZlIn/m7BD5lCrwsL3pIIUogbrfaO10FUhPZcNgbdoh773may1kPVAz8J7clEZNxB5QNsLkxIQWQECFKGVu+fk3C47FG59gqpmLuUHL48Hye9mgesfGIQfjcJJPefzuvFVChsmpKbXcMT0PdtE/nltnf3jyRc/VJHHqXucbZ52qh04k4DfX8sZ3NHXzOYXGW0e3Wi4LTxWqGGULF+vmYJYKBdsystmuWPtd1+LNZOzk00+xHVfsqFCPh8XCc10+bNlVPQh7hDzmaS30NrG4+QgV3Qv77BuF6qLRhQl2otlRH/ZZw95p5MoQymuCp/p/HVwPkx34wxGLoMEkvZq3zJWYElev2PnnX2a1io/M/MrXj7J93rBv8A0eDbDRoM2Nbh3VJEM+n4MLM8nbEL0VL/KNyad5VuSQk5MTPi1AFEpU9f3QdeUcDebvHCg8Fp+FJhKbkL3BgSeagxQzsmVE/160aFjPTCgw6RiIrAAwNI45wI6qE45u4+9iULy0xF7kOvEu1H5h3oEjMEYGQy55n9k5Ic3c49jYhN1wI8BbS4DboYcdZu/6D8Ta6GiiH9mbHdgLVDk4/D5NsiXPWpFcqzcTSKY3mRIwdd655wZCBAe+Zbvttbt95jOfFV4SU0D2yuT4mEvXUtJr1dWbrJp81gk/XoYEvHTtZv5kHbmvPM00AsYoU7oaqgz5fdce3apX2YQOJiCVUqnA8vDGZRY9AjAiRouQ4P1Er9ltd3v22We1+IRo/NxHS2QUIgA+8KV8L5HQgnR1d8nqR42dWMfDUqthvcoGX1BR++f/86TNFH0qu4crZq993Z526Mc+JiaJM6a8zolECRuPmySkW7J4sZeCFhyBFpCBNW2YpDAvu+JGWyj5Qn3ui5+3fV73Wh20vqDsEPNNrpP37+sbCF1CPk6D+/OSmDPLsKw8rBhKcai2jXJxkoI2YzikGAQYVarnBn3l+Of2xImItup16FYHWRzJ6lTKNj81pbEjay7/ltISNjVTDd79/ve2ZUw5zaw76wi4SJ2WNQEg8Sl+LlPD57Ou7im8UcA9QkXAIsaRkJpwm3vtyQMgEa35v2OpCnCKr8iv5fDDQIu1Sjaz571QZXkGPsRtYKDfe52Z3IixTXroyL1jGOJzlKEALESSNwBhQvxDnoih3mWnne2Vl1+W89i6dcxuv+MH6osmGrhszRrr6e/RffAsqQGr8yxwChRthV5q+MVk8gulgiKABsL1Xd32x8f/YD+6//5w/z6U+yz1L3fI+C9avNjxFgFoqGEWpN6CAin16VU7rLD5BW/KUDtoEBfUtI06Rtlr7ZhKjKaMYI/PupJ0zU+/fVqLmTBC4zro2ofHm9GAXt+I7iHYTKB6tGjRihfDHq/jegmJw+FcXuaUer21p2dAi6y2LRYGLeHAuGEzqCVLdL6WzRfmlQ9pYnqrYX944in7x/OjVmEqedpJHb293XbBxav13rOzMyK/C2TBK1a8yM2GIQTiMEUDgbVmU8c69Y03f8f+/txLlkx32P4HHmAHH/xu6+vvs54e96gYEl7L7/tA5pLrUwk1RioFQgnSn46eR+oaD2J7RJjr4Z7UtRIQ4TYVUt4UL+JhlXtfD4vcUIX+YCHLXprzdjYyE1oXG1YpFG12YtQe/MmD9qcnn1MueOA73m6f+txnFa65IcFD08XE8KtuMb1UzlmAwMBByYikQgcMz5CwlvQoKkZoh6UAACAASURBVC+SEkH/43rk+UM+SwgevRVejnyT/LEdjaj5o+agWda7feTFa1V58mjlWGO8L0aDOinhdyy38QxUMgztlLCgBKRqaDrcX+ezc5iV1kGlRXJWhq0ksPPvf3/OfvzAz6SAggG54OKLFFarYSD0BUtqKDSTKELo6ZH+tkcTC97ZQ5MDnq9ldv31N0qQn3Sq0qzbrnvsbh865FBbvGiRX7uqIR5xcT/cg6JUzUT26M3vAyVRE/9a1Ev0pQuz7dIqpU8MF3ltR2hukOe984pjxJwCmMp15W1gcFjaQXNsiNlZhTaEJdwIFgO9IW3UgBiSvHMBXJwslTZnXQ/K8ycHCbBmsLG4CBZLeWgexYox65E19noobJxicd7ynTnbsHGTPfAQM4MIq50yxvuffd43dD0YCRYAz0EzOGmvqHVwWRcKMjQAV4AvhOdszrkANjz6+B/tvvsfVqQxvHSRnXbqqaK+8X5sBJUGRM9DVBxpWK83O83PhdnxRHikeGij4oFCaU2x94ZorCehspPMPeRct26dyi4R8nedLydH+rQ/jzAUVYjh4oSKgLuAWklxEw8wsXWL/f3pv9kdd93vSoL/8i92/MknesN7kkhnQSUdWE0YEAyOG2gOoYumYzGGBwd0aPk5fFueLZ8PgwyDhSdRKae9ocu2bNkyeXEOH69nraenprVmPGcOJNEFBkM0UhH3TfuBCfQYWW/hc2mdhbl5pV4idiDVO+PyLjxfZv8op+WAhusA12ChlE8H3jKLRW7KYRgfH7UHH3zYnnn2eWu0UgK9zr/oQoGp0VBCc/Qw3eWLMKZCxRnNku+y6ZlJIcystcA45FcvXRP6fVMqWR59/LG2eNlynR2+aPTwqMCxE0Jw1aMR7gspBevhDqDiUxOC6gc1a0lEaY4VHG+X9eV3wZCkvf3zOy9poWTAg+zuZS4M9bmqjY2O2+v33VcbbOmSZWHkxBIdZh5Q9DRelHdVAw5jLJ+4En/C6kb4hYQHC+IFfTFjas5jjTKm8sLE9QxXatRsfnbGCsVZe/yPz9qLL48GnVk6+ZK2/4FvtcMOO0xIHTKX6EvR4UHIw0bFiMzMTNnwokUKUdTMQFRAaJdyZHWusGBnnEljdcv+5fX72Be+8Dnr7emVdQUQEQIMUt2ZVyTA1D02NS10WOfIueWQIsWC9RaIIhX9jIwGQEcElraFwV5bFaQfDmhUN9jmdd3jKpwObYV6n6DOoVxTSKvXhefmpm39Sy/ZFWvWqmtqaOliu+iSS7xnNXhcnDYGLl63No8+wxs3+OyB3h5dGznm1hFyYZPR5sACsoEroBtNWI3UC903ArDKJeWwXsP3ZnCF0t09WnvYSbGOT2TE+5B78j0+FwPGSBNQaLI+RNWef/55HUZVPIJUjdaX0D6R1IHGEHPgqDDgxeLEB7w5DqBaKdmG9evUPLFhEyyxhO3xmtfYV486UjVxDDPPyidUeHSj/aJ2vZR1hjY79gRccgTvuL+nnnzSHv39Y1p9bB4O7+TTT9VQcVoNcXC0xHqjjosvSISePxs1vQfeevkOy329lf54aZCcXcYyGCcL9EvO0sycI+g4ocTd153WciZMTioKkCLwZIRBLKZD1ynp5bJBPY91hDDX0eVNBrS4gSTyPbwNYWtot+vu69Wh4X1HxyfaKhiUYQiZgMyxfj29PbJWqO17aapm83MTesB33/ubdkkEz8WDP/e8sx1NTPiB4XdYJEI1RlosX7bMNm7aJMALhQi+6MFkqgB/0lj99NPP6KDv+/rX+USDLMp83TY3O6frrahTo0fhEfTHWAYiJ+MACGCq1rVhooavuocqVX2PA+8lrj43dIEhFi09axQNnyPOHh6367ihruu58fajM32TRaQREGdkdL2dc/aFyqcGh4bs4osusmTG5yU5m6elzc51xQYB9cuqVu2gGpxh8AeBlJq106VNRWkHz8i6cj/i0Qq0c7I94anWX3IwKRkCn0CfkaFns4k1FFBrDvusWuW8g4fmj5WrVskQ4+mXLl2qw6Mp8Gzmri5J0PL+XpGAI0AImbGZkJ+yRgpLg+wMnHPC6S2b19uN199ko+Mzlkhl7OD3HGyHfvRQa9B2SQlIE/e2TWpk34lKSQoHSYTcWuW9ps3NzOi6rrvmW5JaUqkrmbQTTjzB+iBTwGnPgrJ7js6e4F5UbQpG2IFCJvwBotV0b6Nbt8pB8Jooy6soJCDnRDviXTcaqm+zfomf3HZhi2Qez4GahLOjGCkYpu9Rv2V8paBqs6VLlkpAm79X6VlVztohDwOXVA3QeLS5eW3KVTvvpA8Tb7fpJQJCy9l5FDOcUCA9KknB+phFrCULB3+22Sjb9+96yCamPETnogFaPvXJTyjsmZqdbOfXbChH/5LqDIphFtgWjfcMOKZvk02KMr7LdHpLIA/He3H53S73sl09CsM4sPCvuW5a77zX1GF8BmMBiBFCDQzQ5gVwBed2Wn+Xoh8i2v39MkwAMOqL1ZDqzYoKVNjaLjzmgQlIUwdbrBNvk+l0rnGYsEhIXuf6ynbiCSfrcLEZ1q5lHMm2nmoZHTMBdzFiYB0kM9rtE+5A7oiGqNFiMCmXsN4ukOdi9BxoSmSvrntV9FMOD9dDvsyBJ58FB/EWNG86YJPyPKge8EyEnNar+j4HkfQrln2oZvh11drlJF27DrDLFMWUjIOe0cR5fx4R6FODA9GeiB5NO/HkkzTzN9PRYUcdeaTttNNO1tPX3R4Y7kqOrrAiyaTApKKGzhfrRUhOjXfzpk1215136TPpu013dtipp51m3QFJFkmkUhZar30TniPfJ3Xk2jXcjH+Des95rZ9zgKFiD3leDUCFk4K1GAbOC/Nwud3EA3dcJsojJxpuKDeAu0cWJOorp3KO+gmc0OCshHR1N27a0EZVyXFiWURsF3ltzyPwOIrnO+kzdI1eNTGEw0CeGRHJUpEDX7Mli4Zt84YRm5vdauOTs3bvvT9tP5xyuWp7772nHfaxw6ze9HoX/7FZCMuY4aoQE5YLigK1mnIxQDVm4fJvroNNBljGgWKxObBYOsIn1mNqhnqnayBJlLVWdyudzcmy4528tIO0aFZIdjx05Hnx4OKxly9f7p0mvB8Qf6BJ4pkIaeOsIG0+SeU43zcizK7cEL2ue1yMppfEvM3x0ssusWee/psNDw3bBRdeoNEVPDM3TOT/EPKZ7+O90GwqNjk/5PPTGTSavEykdchkbNPGTWp/5N7F2ir7xDoaBRSoi+hPf+yCDCoblmdPuqJul1Dj5hoAHbkeqJSF+TmRX1DHEPIaJkIQwRA5DQ8NCXhcvwH5UydOyFtlMup5Rs2T0JW1wuMT9vLzKOYAAozXQ9HigQcfsod+9ogM2qXf/KbLBNHvHO5ftfgwHV5chihC13R2mdawUbPpiUn79a9/bU//9W86H6z7hz9+qO3z2n3UZonDmhifCCG+r4sojxIYNI8GUQOhsSaodWjPMsKFXJq6c9DOis8+8ptFxAjMN13T3TevbmGtWCQW2vOJpoYUUfei5zXWkLiQqMHEQYSooIG+hK+0e6E5FVrAfMM0BSpA8BfPMnRBKLw2J4uzkbwe6nImWFAWESs0PTlhhblZK5Xm7bbb7rZKVfibVSo+OOsb3zhFdDwOaxQJw5qh37NkyVJHYTmkUTS7s9PDopBfOs3QD4NvXJ8WoMHeoS2O16vUoc4npEUyolYuFLGq3eoBFlraiSbTVtt9993VZM3G5UHwXhxOQs04yYADDW1TTRvULSs++TxeBwupxoXwwD1UJix1EXGiCnFnw5BoQDmMAtfOPbMx5a3D+BR+l++DTQCm0c5HLZV1Fxm/XcpquTHNuNfAC3JPIKWkHfybe6F5RCWJhBNhAFjEpAp1fg4kkQLrRkjLwfJIzCVvMBpEVj4LykeaqM85iBQqrcFwpJl052QYPoP8j+hN0R1zkZnDCzc6TLHHywoQE6vLa+UxR/aupAFhHOL6Jj2i9CgO0NEb1ON+EFspUHxZ73Jx3sZHJ+y7tzDNsKa1xSmccc5ZTv1U77VfZ+TCtWceg8oXCsr52UfqE9cUBFck4SC7Z3eBAHJ9DjYRC5x+rivyHhwHSVjiobvWtBgx6Vxkkmum0TWtkWhaZ65blpzFcGU/V8b3oUyIwvnsl7gQ0VuACBLqxFY9vPHM9LQsBt6GUDbb6eUUwh82EhcDOIQV5RB70/SCWtnoQnns8T/ZY394UkbEZ+Sm7MijjrDBoX4hdlh5HpZ6cxeg5rkFhjiBtYttW5EYTwjiuV9TVpVwn993BL03jNx0obFYp4RiSU9qXz96TS3lwrvtsbcOHR5WZZX+Pv2dz8SzsSasnTwmn1XzLpdVK1c6zTJwwHmAnuN67qoHRT4emGF8H91o7pPnAT4FRsD6z0xPel4ZIifPxXXc9Z6RfgrggVHEuCl/DZJDft39ogyKg02ZLvT9ToyPO5NIw5l9jIlyZJWTvJbKs2PzQaLh/VkDMaVk/NEYg0SQtgWV6FwelYMbc9Kx0VE5Dg6gpjdQmhTYWdckO3jU3DMeSyIMoP5SHWFmL9ex4OXHUGbhPRj+xvvEBhb2AmBoVJFgrahJO4EIMNJJ/eyL2C+LjpYbcP6vZi88/7L94Pt3qwIDR/6d//7vUgrxBhQOPVx+LyG5fDBytB5NxsgEOi1ALfsUI8nzi62ArHPkLHjakdbBxYjLS4f2V3ETCJVFPVOZxiVDlDMglVEs29DwYhvoHxRQ5cBEXhuG36EkRElk8eJFNiutWQcmWGSsI9aHkEYxOpZNbW8UkskvPPTBU+G1hUiHkYtxRg5Op1YuStFw3boNdv0Nt/iUd7G8Grb33rvbRz7yIb2/K/y5BUces1Aq6SG47AfKBt7xoQNLaBg6PVgMrtfRPY82+LtI5gAUoJa8V2fegZaBfk2B33XX3RQ2Tk3PCQySqBh0R4TGOjoEtmGQeChqN6tV1UWjqXP5vELNZ/72jHKZAw84UPegUDp4WylKkJMuLOi9d9xhB3l6CWnLmHhxHw9EM3zMg2K5iAcvFYlgnOJ98dxceSSmF5R+fKbt1PSEDrBqp8H7gETHLi5ycn4WW+AmJpiRO+RhNyywUKfGQzt1Mi0j6sQJBqF7PzHOAQQboIe1IqfdsGGD6I6sNXk/e2l+jqnvPhGANaDUFBsTiB4wPvGQz8/OKn9nXQX8BPJDYX7WwUPCZnAJOtF6eqwz12VbtgC+dqiZgc/j4PBzR++JLd248FVr1tTNdc7Z51kuS9NMwk77xhmWD2NGNGm+XlW6QN6q2Ukq73hzSCz7EYGgPY3zIv/n/tgPrFVspMfAqhRJpBRok3HvRr584kffu6yl0EXuOKML5hdgTnnu0KlGcw+38AqxgIzndC4mm4nQNr4P1mjRcCjF0PkfSNKx3snDQic5ItSEztyItxB6Us8NYZHYaAAuszMT9thjf7Bnnn4xdNI0RXE85fQTdYB4LxElFD7lrVh2Jg8v5nuIgvHwo1wOOTq1Xg8LfTQGm4tQ0nMl18OKXi+WTJRnZbPW09tnS5cst3Taa71bR0asp5/m7U5xlMmXyWy4Hx18wLLpGUH66vrIeWSAl1g0vEQlBUJRSQBpyIELsRNBM+aRtePhY4Q44MuXLW+XimZmp2XdOS3IikbVB5rGly1dai+++FJIKZhQx3QDrw1ivHRdMzNyy0ReAuXI18TbriospguM73GIQUmdUFO3gaFh27R5cyj7lLUPCGPj3CCfUuDaWy6iwExbryQAYIk1lUqqbs+9EplheOMeoPWPgyDEP5AyOEQYNcJhSRmFEk4k4uAE5DWpPde2TUXwkR5uuB3xzqkzCU8moCkSPJQmecSDSotmBYEnbBedUY3AmOy7776qj8f97Q0S6GA5b53rJudXX3Ag17A/XEklODmGdisF9W4wIpioxhFHjjhD0NMYnAlGIfGTO9fo4HJx3d1O78NS7LXn3vb8Cy/oge6wYpVYSngvXudzQJFc8Q6N+MEsLl/Qvcjv1LIU3o/F4CZk9aQ36zqxWCfek4VAw9fbmpyxFRX7CbXGx7bahvXr7ft3/lAaQlEB4evHHBXC4G7p82DRmE5OO5rCRw3faijnJcSL4SgbSXB+AHxY8CgSzsPn2tuatlGdMqh3gE4K/at5SEoIjbUXEIaIdtWjDv6LFpjPldxL0eVNRbHLddjmzVukErF8xY7aLNpMKEKE+jDX5F7B0Wz+zXpxSLhHDgossfiFCke0ypk0RsjRejYGUYd714ZyWIw1hjmG2Zo+MDCgtIEDTJjHsxDxXjUNJgV4OZDfLWqcqOsBA0Byb3wW6ChGgGtWjZRDgAcNhA48KgPbuA+tSSibOTjjmtwcYkTiXL+Mg+sbXDgAZSd1yczLK0rOt97QgQc3wdBzTzDhRIhI+GxaB5kQ6+/TKBLXE4tSMj6GlahQTkpcdMLcbc0RGB7Wjb0TcQOF0YFJxnPaHvCKZdLI6WfdYq3Pwc1SEJh3iSYdSPjQ0qqecVVNgW7cs5f0MEhCzR+860qhyiwKibv3vjKR28EPFp2DouFJRW9aj83vxP3KS4JiIIuANaSlTAJe0tXJtlvwonypfr/sdVEOKEgvB3ZoyBuL8XYuadKlG2GTzk5PaF7tj3/0sG3ZPBbqmGY777arfeLwwxXaU0cjFOfArVy5wjZsWK9Nz6FsAzZBYDqCZzzVqE9E2KoNWSyqiM5hZD0wHJLHIT+kuVoHOWGLFy1ViyH5Oxt+enZGeTqenPVkU4Im8wBZDyHdDdMDIb9y8GdE2lE77bqL6nkCVBLu1UFcIyuJa8IgRuSe94ujKXffbTd75dVX9bO48dXAX3HJVw4qa07aIo5w1TefRlqG8TNCzK0lMgThN0Z03br1Xr5iHAeT6oLgQQxdKzUIFA44Ue7ivdjYTmllH/kAa/YQeABGZK+99lLoSu1206bNttPOOwmEZG3Gx0Z10GNr5NLFi9spSFdPj6IRIhUiQYnei/bqbYkC7wK6z3uLRgn9NnQPRa9KAz7eGULN7KzvUT+8pAwdGvki2iRRaMajnGiQKOdg/FlDdSjh7cVDQD+cUlVJRhtjvXnzqK1cuTJQOSHpIEAxrOuNnykuROhVdnEAxoQ6YwyHE3W7uGfSCowv16gJgb+8/4YW4QCHgxonb4Rbh7/sOkD9No/anEYzFGzVyh1tdsZnp9CRwYIhrk1xmvchNCMEpMYWSQexw2Nqerpd3iCfYXH4fTY+D165cbeTGTAQgDx4CGiKauFutmzdulftttvucBCnRY9qhx1/8klqII+80wjD8x4Io0dubkQ9IwiBd+MhRBTVhejo/3UpUg1xDjNq2HRxTi6bVSGX6tg+uY3rQL9Xqn/kcINDAmswALxGiGc2o8OD1+JgIYvD/XPoXrvPaxXV8FpFMEGtYnJqQvcVw2hCcA4HXVQ8bCw4+S/q+9G74X0U7klQzdVFuKb43soP83ldM3+PKUZPb5cT+pFuEartSK84y4FPrWpCt0/Ac8wjpDZdcNgn9Yzo2WXTxUPFvbJxd911dxuiHFepSO+K+q16W2HepQEG5wOg6e2RFP4j7ZG1IzReuWKlHAHvzT6VMlGYmAgOgdGMaDH/pv6u2VdxhCXRkLrbnCQSw1KtF+iwaKeek1Ka4nDJmAZhAO4PcIn8Wg6ICEo9x3hoz42JbMi11WJIWhiINxxMqix8eQTgiDZRCgdWbYQouYSxrDHXJvVRjblU0rlQBPXgXWs17JEfMmaDw0bdjgiSjckCLlqyRHmbtGeDcgULNzDg4SgL19MFAr0tN+OwKZfr7DSQSQ1SCiUPLG5nR05yJ5ETDMghS5JMS5+KjQ4QRrsgpG7lK3i+uXm77rrrbXYWhUGsedIOPfzjEvCW6DYHIoxu8PCfMNbHo/BweN+h4WFZbLeqHpoJYg9av5QuhCAX5uW9o6aUPGYYQA1pgXo03hgQig0/NDiszxCPWTNnMj5oOekcWWp47Y3AxMICD6JPv0+3kbScQyfPyJYtHq6LMeRDwvldlRSE+Pq/QUoxMG394qBqyIPm9zTLdnBQFhsSjUJfGSMvufAesSTV1+dT5CIUHRlw7A1KGD5Hx6fIybsDGs3O2dDwkM3NOrWU9+rp7fayYhN5Xu8K4lDw+0QNdOzgtdk7pA2sobqOJNnje5D1YCPLcBRLEmEgyuAZq2MLKSBCaqiFAQvBAPMzyCGUsYh+hhYt0s+5T/SkWb84PsSBwKbjECE9QpdK3lsaXdt0sajju2SS66ppRE44fHymIkzhDN4pxl5irSgDqsOuCX3WAau4jvw75tMKuSW4j8P0hvnwIByFl0H3MTgY5sRDP7i6hfWQNEkYzSE91xQ1NBdmLgdVR8KJHMoSaBgpHNqmESw1Wak0kB/5IKyYL0dPR/4QifiIzmFR2ORYEc89E6Ii8n3AF7yTwnb6GFWg9+6O9es22g033KiDy3Xstuce9qFDPqJDyesxJEIc1e/bLdYLv4vnhfmF5cMo4AWwum4pPWRSGCMFyW41PwvoYWg2k+rVweG9sRGaj3kb90hfaewI0XCpICbg1txRXB7qDkxKn5wUQo4n5GHKC4f6Kd7HqY88yEIbrYWUwOt5ba1GiOraw2xijMhee+8VaIJ0L3W258KqZS6Q3rlu5U9C3D2EjnnqwoJ3VLHhhgcHReoXaJn0/JTckL9v2rxJhwKjBm7B8xobnQhlvLyaNYi4IjhFXVec5Q5+5iAi98hhxejwM0UGAJzq06WcBxMqKfaW5GOQPgpD1+ANq8QVOMbq2qrVbXxivL1vqFZgOGhIUCkmcAqkpIEqxbR3v3H/S5a6QDkHgrlUQoMVBi+0CUYQhiKRBWejkmkcQK7JGa61jcHnekhz+LmrdlAtIAXyPNq7rIhgQZgH5ElVsgyCfP5zb1mNgC5nkjIlLlZ740d3rRWtQ+1wuS7beeedVfoZWjSsXIcL2mGH5QGE8lYpYnh1uaBYqLEPxOqeF7CAeEM+VCFVyXMCHfSG10yxtj5P1DWN8N5sNDYNrB/EswA7IDJQVuGiG1JzNL0nr6c7o1Bgoh+AQtbO+MYZIrqLtSUVDpBP71DR4jFZjsgAiRwAjyCu7rQ838hCtfPdCpVFZEDnCKUHmrYVevqBEmAQh35r4rlHJhIfQENYAu2ICvjDVWjOjJsGEj3eVifBsKAjrNqpwAlv0GdTC6lX3ZgGBxcOJ8Tj/nzQ1oz+zfswo5XrwZsJIBGxH86413H5TIgo5HYoNsS8LZZ9eE3cILxvDKnVgkcXF/cS7hFjEUE/nAI1WIwk1xvzY1InDoL6o1MeNRBOUm9n40oNEo9a8vk/UeKHtcX78W/xAIICKN+X5GqvixJiANmv/eIf0KGVs+npMBKF0SYFat2wAEuaOhDJPSDYqslLnZS+VkaXIL/TbHPlNYw9MLCoHEiONVQSeD93DC6JxLPCeVHFYE3c+Xj/bDrp2loe+XjXlzqFqLA0mzJSNLrwjIXgy3i7cCLVEkWPqFVmaOlzuVmBjkEuKvHLB2+R4A6bhXsBIMITkRuwkVhIwjLfbJ1SAwC5w7tJTKtUbBPzuSlp4LYSYhXFRgNyMg5k9KocRAe1PJ/i4rE6nrT78CbAEfIVvg/ZgfIU3tNDu5r97OGf22//91HrQHIllbArrrxKVpmNKzkSych4aB05tHgnrCpGBoOiujGjKygvhEK3y6Z6mYTP8oVPKa9nLbztzj0714HCh4d4zmwSQ4YGAwmm+b1E7xb7TGMvLNeJ9Wajq1QRuLh4FvIcrsU3LTK3PodJXNhSSd4KY8drXQYXxpnTL32WLlGE58saZyn03NUjMURisqWZBtEVpIjmJEbA+hMBqbc1tEy64FnSmXIqw3h+jXAbeSnXHUdv8nPqvoTD3mTviv+xOYBoTTKooUnC8zwP+1U7DyguOTTeFnIPa+NtkhhJclTPodk33BBRCOg6ObaDe3QU1WS8aN8B5+AzyIcxBtKRAmkuV6T0GLEWFhjPiuHmnoeGFjkmQVQSJivKgIeZPy5BhFekf91VXSI4mWx5muYgYsL7xoOqpXdlIcjrdWM8qWYFB/4An+FVAxp0vOEj7jHuT/nxQ/ddL7E4z0e7xOkdGxu3WsOJ2yIwQE0MdDo+Tq9PJsRo0thCrAxhRo55sj4NnA3FwWEB8b54Bw4zG4mDy8YUZznr8iLcdERteS/4qBw0DozXZZ0YEnPVjRs326233i7k9JjjjrVddtlVjeNC5BAOr1fbmyl2qAA++ThFZ1nxYGP5ieuIvN/22Azau4LeMg8ecA1LiYohm5V71EYMetLx4Ea1CZVUAuvMx3e4mrD3ETPn1g0J60kTOgc41lEVSqK0wcMLYlAYMgwe+RiHjlyIPx008zICmxEPhFHU7FhULTTp3SsHkSnkNUyPZvh81oH1xVizB+L0PDWHMMAKemAq6XOLNMmgU5I2KtWNjyvSYLOxyblXZxOlbMuWrerUIvrBA0stRU0DaJI5zZAv1oTDzwaPVY5i2BdqGYRFFsp9tMPhXFTTDFPsYmTDtXmNtyED5IJ0/t5DADtoVhtig56i8bkcGtZIrZkBp2GfsK54eYXqQfVF7LpZF4Gjvc6li51Drbp0ULFs1pqqKAiwQygiGHAZIZyPKMNet5ZHDdROno83y4Qh5DRjhDWKfdPKoX96zzWt6HUAZXbccUcb2Tqi0JTNIIQxlWz3XjLyA2CGDqKF4pysOUAPelIuPpYSUBU5n4wSwUqSH/T2+CK0lQdCH6iG+DYa2qSEyVE931vtAHdQcHBBMy92t5x9AxId6m5sLLV0wX2t1qT4wKaK6vn8HpswCrv7FDQPPWMdWy1dMLNc9E/DpllUQhgOY+Qts/h4bTa99KBD0ZwSmvjWGtTkuk78G29AOAuiypsARsVGc1BJDAgglk809IZuNj2bAiPjh5v8qEMgDcCLG9WGjElku4iGlAAABCRJREFUHLkAuAOCfPEMYo/00CDtmgsqW6E7heFRvbzF5s+rrEGP7Z577hk4z82gPwUN1u9TG0rDnV1vC8EC38hzWicOBJES3lLtckQIGRc6wGPCGHIUviBjHIEZ1p/35plyT55z+8wmx1JI0SDZZJ1LHTqzWF/RalvNNjEEZxD5zUSJpD7kwp6COKkldhdFAAjsAqOAB6fCwXrwGsqjXBdeE2A1aoJTHpXWVRgMx30IeAq4DYeUZxpZXdS1Fa1pjlVZxoQoTPsj7EsYdZLMRaww39XGROJ0DHCMOOlCketvH/quDi5vitQpC7t1ZKs2VqzR0sdIvsfDQrGdiyT/heaIM1CPJ8RtwBRCX+b3dNMSZ2pWANRyDm5SHov3jaJx5DtsClfLiKJrPkSMDaiQubAgYbeIytH4oOFJ2w2X8gHEAC/T4X2cYeJe3bVs1RQQCtqE+NLUCg8yymCqplz0MDpuEq6L0hSHlUNMjiTygggGSK24hCgbS/U2Sb26zjSGI67X0mXL9H1J0kr42r0NuIAMAZpcMnquWQyAETm/fJ+p6q5i6WU0hY9hDWJrIjZE94JiBV40IK4uyObPis/HoLjXHNc6iElWWNDrBdIlgkZX8BARVCRS4Nrd27nqSYyEmNTI+4JLKH+UtIxPvZDHWzTsQGMwyBHg4/f5OWGyWFuBcBCVDsWTDmJ/3D+godD08F4YONoo8fQu8ufKGbyXUsCQa1ZDjdm7pHwNJRUj3r3rb0e+tOeSTq4gxdH0yNCdBHYgrAE1yaCGKU4yfduhm4jzQmUF58L94d2JcjylcoFAOZogX4tmG/tAEj9MhdBEDAeAo5H2PdzlQnaP/eKOFofHSxcuw8ILyJvk7eBapn1GEMVyFCAJpTX/pVbWJlfTr3RnAy+YDRAI77CMsHxCfFM+uJeNF9viVOLo7fG2qqSDEIAFHAoWVaADjQ1dPdoIKpHUnZIWPRNWnwdFQo/VxJjMzdH0H8XcHBRjcxNe6nfDOA8PXbzkozpynkZ6R1Mlxr7dRAMvo3iow/vBPeazI9UzDiMTN3e7vC0CRmIJBfqjxAoS8KN9GBjvx4Fg8xEGUq/F8OEJvdifkPdQTTWQBoRkS8PJSxO8P/VRwMRRGq41+DuntVdOzGiZMJOHDeKAYU20RaIdZzT55uKwSQo1oL9+nWnV2+O+KFeK8q5qpaTPFK1r5u+EEFe17c5uB4OIiOgiChK6sfwTh8Lx3jxD1/XyWbWUsYg08Oisgat3NCSBxHvHvJjXy6BovCtRlbf04RBE+glD0/g7835cAgc8Jsw9qjnlF1AxVkD4GSArnpUDRB0XY6TSHNTgJFxjIifmCnmDCsqP8fBHYJFnuXLFCj+ImYwOL85DVMjQiKN6MEO0Z+eUQjr0FWq3lZKrcbAuoRWQn/1fbh9VCp+xIjgAAAAASUVORK5CYII="/>
+        <xdr:cNvPr id="17" name="AutoShape 9" descr="data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAO4AAACzCAYAAACO/iALAAAgAElEQVR4Xrx9B7hdZbH2u8ru/fRz0kkhjRBKaNKkKCjGC4JSBEVERLkowgURFDF0RQREpLeLqBBCk4RAekhIAukV0nN62b2t/j8z31rn7ES8/733+Z9/k8Np++y91re+mXnnnXdmSXNef8Lp7e5Fe9GE4QAOgIDfDwUOZEkGJCDoC6JarcI0TehWFY7j8MeUFgVnTWmE6VhQIYOebFkmbKsKwzDQ0NDAz7MsC/Tw/u6fvpZkSJLEz4Gj0v9g2zYcW4IMFTfe+Av4/VFEY1E0NdbhlJOOQ1fBxt7eEtq7OpHJZVCsaNDLVew90IlUfT1s00IoHIJuWDhQigDBekh+P2RVhRrwIxQOIxAI8HN8PgWKokDm07XhUxVIsiQ+w8GktjiuOi6C+qZ6xEbNgG6GseCD+Vi0aBG2t2eBUBKOraOqaTB1Gy8+di9kW8M11/0cPUUdtiNhZEzG9791DqyqiY1bt+Hj9Tthpy5AJpNGqi6BUqkMNaDDNC1IjgRHTmHbrl3QjT4E5ACi4QiGN4RRV59EPBFCa3Mr0uk0FFnB4pX7kSlbKJT3IKBYsPQOSHYJFcNAUFExcdp3MdDfiaOmTESxlMX0KWPhOEVEohYCko1oMoU33liBbNGHxi9+CTvrfbhg2hh8eKCI7v4sUqYExTIxkOuB0r8XqR1zsbXhHBx53NGYEMlj1iWnwDJN7Nu/B3975wN0ZDVojg+5ni7cdPU3UMz04Y677sT4YSMgWRZUWmjLgGQDsB1ICqCoKmRZAiwH9B/9oz1A14WvigLouoP2TAH5ShmmBfzp7p/g5OOnoVAoIBwK0VblPSY59Fwd5XIZjmTRbuKtJdF7ObTDh/ai7dA+Ez/zfk6f6eeSIiMcDvP7K5IC09Yw85qHUDT8fJ0cxwb9pzgWTEnBV49twN0/vxbxYZMB00CxWISq0N7y8fnRsRm6zucFiXaWeNDep9/9V49B+wAgyzKkt2Y/6WQyOWzp7Icl+wcNl1ZOoSdIEhTYkBUZlUqFl4CMk96IDDlabsdV5x4JRRGLrCgqLFODrmmQZBmpuno+SV4MOuBDFoh/DmnQcB1bGXqeA6z8cAU2bdiK5uZGdij19Sm+MJFkE/Z2Z7Bu01Y0NA3Hph17kC5U0DOQxojhI2HoVWiaDsu2sb8UhRRuhhwIwOdX4GeDDUP1+9h4fT4VqipDVRU4tskGK7MhO1AkCRObo/j+iTGkGlIIDTsaVc2PVatWYv7772NvXxGGGoVtGqgaOizdxnOPzEK6vwO/f/Ql7OrNYlgqjrOPGIZhbY3IZ4tI5/uxZ38Z2/om8xrGolFAlmCaVciSn51OxVSwcfsm6KXdCPr8GD/2KMiOAUmy+QOOBU3TeHNqcgTxpsNgWXnA1mDpWSRiQYwd1YrO9n3Il1vQ3t2JunAMra1taEj6AElzHYSDukQMjlXFTgf4bOJR8KlBfPmweuzsyaKnZKLvQDeGNw9HKGhDzqWRmXMPIufciExJw5cOT+LSGS1oSiaxp6MTj771MYJ2FkeGu1Ep5dE6Zhq6s2U8/sRTmDxmNMjiFIlOlyxTGJktkbMkw5XF9w6d39Cm5o2tSKjqNg4M5FA2DBiGg4WzH0V9IohSqYRQMDj4N2SIWqUCTdc/13A9I6H9WPtetYZLzkPx0f7ws+E65BYkBV/+3v0oa2T4Yi+zgbNhO/jzHRfijDPOBoJxGOUKBy+Z7Ef187nRg+zCJudSY7i1BsuOxwtiroNhh0bH4P6Ovpfefv1JJ58v4uOd7TDVAL+GLCu8ib03U9w/oMhpOxYdNUzLgmNr+NrkJIZFyogn42KtHREt6bmGaUJRfUgkkgd5udoFOtRwLZN9ED/f0DTMfvVVpJKNqEslEYtFodBx0YlJDjp7s9j2WSfijS3YsrMdhiWhUKqiohniojkO9GoVXVoEmq8eaigGf9CNsn4/G7DP73MdDtiAySh85IBUivw2VFnCqKSKH59aj1R9EuERx6JcVbFyxYf44IMF2NOf5WhuGQaqugbTsDHr5h9iTHMdHnr8FazcugvHjW9GW1TCKaedgo49e0ExoD9Xxd8WWFBVen8/VCXIjpIcBjmPiiFhX2cnejvXwjIKOGnGOZBs2gAWorEwTKMCmyKF4+CzzhyUSCtkjkwyRxafIotNSf98QN+BTWhJtMA2FYQiQQQDYcDRYBsSHLsMnz+AhrNPRldrAoVCGjNGDUMoGsauzl70lGRs+7QXMnQ0+YH4wt8j9MUfoGJJuPCYkbjy9DGQLBu7u7K4YUEPDi9uw1H6CoT9QG9vHn2ZAhas2o6Ro8bCJ8lQJQmGbcCxLMgOIKl05GDjJSPwHLzY3IT8FECVkC9q6C1VUKjo7NzWLnwRsDTouuH+rRtJbRvlUpn34OdFXEZ+9J/tHGS4nhF6hhSMhNiI6MOEhEy6iAtveAqGwZtUoEmpAtkOwIcy5j9/PUYefipk1YdiNjcYSQOBkIisAO/LweD1OSGWtnZt8KX3ONRw+ZjemvO0o5eKWLvzADKmD7Lih2QZcNjKIUI9LSihGItgnA4TCvyOhiObwzh5HCAbOi9sNJ6ETl7MMGFZNgxDh2QbUANRROMJOA4ZuwJIBrmHocgqy3ywtkUeTHhdOuAP3p2PSCSCRDKBcCQElY2JsQW/1qKFq2H7gkikUti4uw+VchWG7aBUqqJa1WHLEsqVKhw1ii6jHlI4igBB5HAIql+F3+eDSh8EiSWJoy5DZFlGKKjycRBSaw368NMzkkg2tiA+9hhUKj4sW74c8+fPx/6BAuxgHJZmo6iVYRs6rr7sApxwxOFYsHgNnn11EZriCqaODHO0PebICbBMA7v3d2PJOh0FNECFClMvwbIcyKqCgBJCsVpEpH4kdu1YhkppP5pSDYjF63DFhV9Gb18/PtvdiXK5gmAohO4BBUZwNPyqCsumjUZe20E0GkCpWOHXHejajrp4HVQEoUoyTNPgcwUIIZl8/kWninG3Xo3S/t2YOmk8DEXCZ305pNM6KrqCge5u+GIJNMx9APqkmdAiPtw+82hMa9QwqmUEdnXn8KNXNiNo5zHSOoDj5U0YGMhjIJfHkpWfYvSEKQio4Iir6yZff1Wha2ox5GenLLsGYVJEk1yoTNtFQrZcRW+2DMPUeS+u+eA52CahP7DToy/IGC3bQqVc4c8SuUk3Onohmd6XIPOhhusZI6dpcBBLJIZMyzbx4uyleOqN1bAc4VzYJmxyNgZGNIbxyu8vwvBJZwOOD6V8cdBYfX6K2oBj2xzMhgzXTQ9duHxoQKu1axGFh+C09I83nnEqpTJ2dfVhX7oMS/LxG9hsHAJPB/w+vrDk4WWJFkNGWyqMeuMA0rksdn66E0FJx29uvgQWG54wStMyYelVmI6Ozv1VTJwymhfRkil3FHBI5CQyDIMWmAxXZMtbt25BYSCD+vp6hCh/USWOtF6ebNkm/v73f6Bp+CjEonFs2NODTDqPctWA6g+gVNLhyDIqlOtUHKT9bZDDcTbcSCwK2afA7yeHJENRZAHTZN4f8PtUBH0y5/h0nC0RP244I4mG5mGIjjkKhhnCwoWL8N5789CZrcAKxmEbQKlcZHh03lkn47KZZ2PvgTRu+vXT6Ow4gNOPGQ6fz0HE7+CwEcOQTmexaUcPDuTGoqrpkNUgZN7EMmQfIQoTajCJYv9OdOzbgFhYR2NzE1qTEVxw/plYt+UA1n2yw82f4tjZVYaqhGHLIYEiZAWOJMPHMM2Hgd7dGBjYiqAPCPqTcBxy7WLj0LUNBANwNBNj/u1ctE6fhnFjD0PBtNGXTqO6rwOObaA9b0DzBeG89zSGn34xtvRm8eSPv4rprT7eFzs687j6r3uR8pvQynlM8OUxrOt9+FUFz85ejCOmTEDYrwjD1UwOQbQfac1p/RlJ0abgvUZG7RPBw6fCtG30pHNIlzQOCC1N9fjHK79DtaLB5/MJjOZyL/S3lNZxoIEFmwy4ZuMLwxWG5BmLB5+9/UVPD0Wjg7CVHOH1v3oaa3emYdrE8QjHQq9jyRK+f95R+PGVZyI54ijYugWtooljd1MA+to0DE7dPCjM8Nt9/N/y3H823DnPOJWyhmyxiNU79sEORGFYFixb5Ld0IsGg8Bj0vSzRgquQLLGABOvWbViHancGC5+5FgHFgcMeX/xtuWzh+p/9Du1dFVx2yRdxxcVnwaILpci8sLyIJkVb4U1sKCBHsmnTJs6bgsEgX1QLdBHEg55pWQbefON9JJtaEAiGsPVABu37OxGNJeFICvoHcgypOrr74PMFYDWMh5JoRDAkDJciLm1wzuE5n5XYcBWZ8hUJAT9BOkIHNlKqg1vOaURTywhExhwFywxj6bKlePfdd9FdqMLwxwEDKJbz0EwT08aNxi+u+y40M4CvXPgLZPN5HD0hiZZWP+pSKUhaGU31dVj38VrsTsexZdNmtI1s4Yt64EAHHQRikRjidcPR2DgRDQkL06fGMG5MC1paGtHc3IC/vTofjhlCT08X1m/egZIdQH/GRDCsMtqhTeVXJRBMI5YiHE2hr7sLo0c1YOP6tUzYsHGoAeYi/H4fZNmGKsVx5oP3IkBOLRhAbKAHxw68i5FNCV53XcvjP19ZiONPmoGGuhhOPOdCdGUqGDlsLLLpbmzZ1YXOTAk7uotoVVU0GxvwwdJ1eG/pGkyfNgXRoI8Nlxy1iFoUBhzeD2KPkVEIo5JlkfcyWaXI6BzIoj9fheRYOOWkGXj0rh+jWCrD7w+IvUEGBQeWaaFULonXc0R6d6jhEkT3jJQ+e8fiwXQ6nkAoJN6fSCjbxDeu/QP6SiK/pSAmILcKWSrh+TuvwCmnngwn2gSjXIKpCV6Hoq2XchInQScnzon28cGG6x1DbaStNeyDI+6cFxx6wXw+j1XbPkUBIZiuN6YX9zwhQUpeG9vkjc4naBv81rlcDls3rsG5R4zAb/59JkcpQ5ax89MO3HjLg6jqfui2jnAwgCsuOR0Xff1USGoYNhm4ZUM3CbbQK5Gx+HDf3ffAMmUR9RQFyUQCDY11aGltRENDHSCVGWqt3/AJLKsevkAIn3VkUawa0C0H+zu6caBzAGogiGgsgT3daQSaDkcw1oBgLMS5G0UYiqzkrdldsPHK7HRoC8mSLTavLCNoWbhjZhPaWtsQHX0MNDOMNWvWYM7rc9CercIORkDeqGIUoVdNtDbU475brmMS77SZ98ExMrju+2fh+GmT8Lc334Bsy5wv+n0h7O1K4d0P/go4Oh8T5dm6XmGSLxCIYerkmYDUjWggjRt/+h0E/UFOXwgmd3QeYPZ007Z+PDdnCzLp/TD1XjiWAZvRggk4ClQ5iFPP/A5WLF+EaUcchfXrP4Bl98Mh1FZDhKi06UMxfP+Rp2GnGnlNRvRvw5HlZYgEAwhHVISCIa4weGzvmKMvRFHycVWh78AO9H22ktezq6sH7fv70JctYf2eHDZs3I6Jk8chFgyCAAXBWK5a8FoLR885JuVvFCdti9MYj4El8NrZn0WuojH0v/m67+HbF5yOYqnAzp1gr8cq67qGarUi0JxrIl5kpc3PP6/Jb2ujrWcojDTDIjclY9MNA1/9wf2oaH7QVmXiSZahUOrns7Ds2e+jZdJpUKQQCoUBSA45UMtlpcXL0LWqfdQa7ucZa63RikA4hBCkd9940aGDIGZu+9792J2uIhiNI18sD7JYnD9wDkjQcsg7yQx3KQoDH320HAFNx7Lnr4NlG1i6aCneeH0V8mUdVd1kOFhiRs3Ed751Fi666GsMMYjrEnmKgObLl67EiiUfApbId8jzOZaNUIDIJAXRqA/1jQVEo5R/qEjnYgj6QujOGXh35Qbsbe9DIhLD2LFjEI4nsGnbLhzIO1CSwxCIxBCOBBGJEUnlRzDgd8+JclmBMCjvo+iryjaTPcQkRmQHd3ytwTXcY1Gq+PDJ2rWYM+d1dOU0WMEoHEtCSS/BMYCgLOHxe29lVHD2hQ8iFAihpa6Ec04ehzETJuAvr7yJdRu2wLJUnHHmJZj9+n/CsEqCA6B8T6GNHMDxx50GvZKCjh7kM/tw0w8vwbhxTcTxIxJOoFQsorOrHZt3FfHsnA5kB3bBrB6AY2XhEPPMgddBou4whCPHIp85gKOmTcWqVe/BsnshgQi8Wq9v4oSTvoThF14Ju60VMSqNZbM4r/wGI61EIopwKMjGRAZsWjZGH3UBuopVRPwhdO3ezIbbN9CPnp4+VMsWduzpRE5twOqVqzBlymTEwkE4xH0QQeVufoLSTKR5ZRoi3QjJ1+xmw7LRly8hUypRpQXP/PFOHDd1NEdWMlwRcYVD0DQqRwpy8vMMl1/ZEsTUoaUgj7kleO4nppqDlYWiqeC8q38LnegZm/JziqiCT2gIGnjz6evQNvF0SE4A+VwfVMnPTt/jZWzLYkL3f2O4IuqLGO2t0aDhUk6QzuexcnsHlGCEa4CcIzA8pg1NueAQeUAHRAYlfCYwMNCPLRu34sGffAUL5y3Fkg9XYFxTBD/4xnFQ/SYK2SoyuRIMUwGR180jx+O4U06FYzkwyP4p4beAmd+6FhWNDlCCTBfCshGNRhAKKQiHA8hmswxnJRAEUeD4FZx53CQcNnY8Hn7+TRxx9LEYPXo0ksk6xJIprPxkC95atBZWKI5gJIxwJIJQJIJwNDxouGSoDJU54eJ/8PuEU5HIcCUHv7mgCU2NTYiPPQ7lagCrV63C2++8jfZ0BXYoCttwUHEMmBUTsmXixT/ciXKphPMufwTZHHEGQJiIp7AFxwxCkoKgYF8fj2Lfnq0wtDwzxQ50Jl+IufzmhZdh4/pOpMv7EAr5UBeuw+XfPBqpxggTTMSyU2R55fXVeH89UEjvAcwydG0vR3AyWhkKxk8+DwN5BY6RxfRJh2P5h+8CKMD2nIVrNFSrnDrpTGRDEQw/YwaUxpGYFtfxZX0hfD4LwUAIkbB/kBfQdQvjZnwLOUuGrRnYtGoxunYsh2YYyGULyGbK2LanH+VwK3Zu24wxY0YgFgxAdmwYZAFknLbNXEPtw2aoLwgpLxoaFtBfKCNdKDCBOeeV32FMYx0q1QqCQQ8qi/JMuUxEnyhZ/k8MVxgpQXSZ0yjVI5UcG3MXr8Ksp5eCDNCrnBA/Qsjm3uvPw8wvTUW8ZSpMXYamFSDZxKGI8io9n2yJUqH/qeF6rPY/Ge4/3vxPhyhqgsvFQgGfbN6BPtvHxIa3aH7Fz19zHkJ5oELlIsG6eqUf2ZGxZuVHMHUDl55zLK6//EuM9Z1KN6qVKtKZNDID/TCrZfhVGUEiqIJRjD3meE726QA7duzGe6+/jkJRh6P4YYrsBrFoDMlEGLG6FJcT6PndPR0wDBnwJ5Cqi0GzVVSUKKKJBLPb4Vic2dLO3jR+9/SbgD8GNUL5bQzhWAThcMhllVXOuchz0jlRfsvVJoYmJp9zQJVw/8wWNDQ0InbYsdCrYaxavQJz352HfdkcDH8CtmGjajswqzpM28LLv/8115Kv+dmz2LSryMgkEkkg6Bfwj6KN6iM0YbIoISL72UkRdFdhcU5HHrp3YACSkub6X110AlQqwTJBSLyAhWRdmNnskjQM7fu3wC8XUCz0wrAKgK2zcGD4hLNRzNporIsjEVexaeMKhEMqKtVuEKwUD4KpKUyfei62bfsQM0b146YbLkYIKnxKnllbZuOJA3DJvELFwLgTr0C2VOVIt/wfrzGZVs7mkS1W0NWZRY8RQFaz0NXVh/EjmxFWVdiwYGhVvrYE+wXxKQzGE+uw3brf0/OqDtCbLqJUIi2BhGX/eAqRoALbMvm6kQPgNbFtlIqFQeKJN6kLj5l7oW9Z3OOWgtiwDgaq9BpUzQAhH0eBQSjxlqexp6sA2ySRzJABUgBe/vSPMGriZCjRNujEJrvkFeXe9CAcRdeb7clNTQQpO0QO1gCfwYMZKgV5PyI7ETm39ObsFxyCFSRWoGL+nvZubOvsgy2LNyXoKFFdlxhPiS4veUg/wxOCuLTZaAMR2bBl4yZolSoOqwvhtSdvhc8JsKF7LBoLZajUxAdNsMHi8o1eLsImn0BMo15BVTNQqlSYVKGLwlAl24mBgQHEQn7s7yshFG+CpgbQnzagBMjRCOaRVCrJVB0Un8rOiC7nDb9+FAgm4YvEEXYNl45fCC9UdiSKsF4mSjzhCUt7HKrrAg98vQ0tra2IjTkWphHC0qULMX/+BziQLUL3JWCbNsqmBVMTkeT5+38JvZLFc68sxe+feBeRSJyFDcKLEyynPFeFY5oIKn6komHOa5nIcCReg3JFY9hnoxO6pqOx8XD4fZQH+/nYy2XaNhZylSL8yeEY2SzhxceuRkXTUSxXUK7o+GxnN+56aCkG0n2ApaM+kYJjlZmIAqqQ5Cp8ATp1A4rUBFluxuYt7+DbX6jD5ecfjkgsCVkRiEt4NPcYAZR1C2OPvwIV00KxVMLcv7+AysBeFHI5FEoauruzqATq0ZMrsUOvT0QQpCgrO7BIrOJCR495ZUEEGZXjCHRHXArVYh0gW60inaf10LnKsXzuU7BM4gmEIkkwWsII8/ksfy/qwHSeLpHkGS7tWfd9DjZZfia/XiQcgUOGa0msirrkhkexr6cAIgYIGXqQmljy95+5EiMmnQpHjaCSyUNxlYB0DuyU4HD9VhyPeLBRDuLVQYL/0MNhJOgFULZHlx2X5rz6rENJM21yqn3mixUsWbcZlhzgheMnkkzQ3VSkcmEP5zgI+Ag2CW9JBrLr08/Q19OLsKNh5euPspqEuTPXy8jMwokDIWN0qKxNTsiWUJUcKJTbUCQmL6dbkH0+UViXJQSkAG6+6UZU8n24+LqfoOyQ2siBZDgwbR2VquYSHvQ3VI8G18wIkl13+28hh+rhT9QzxR8Mhxl+E5PKG4QgJW1OVomJTcPHLAlYpCoSfvf1VrS0CXLKskJYsngB3ps/HwcyZZihOi4BlHQTJknaHAe/vvZyjGprwPtLV2Pb7j5YpgPTcGCYFtIDWVTKOspGGZV8EX1d/ahLtXA9WcBHKtTTcx3ouoJYjMwzj0J+AKbhhyrH4Q/4och+2I4BWY1AbRiLpoiMvz75HT7eQECFLSnY9lka37thDnp79wOWiZCa4DTAz+UuujwCTdF7F/ImLFTRn/kYt1w0Aqee0IAEIRN/lEk7TmBk4jkEE7+/ewDTz7oWhaoBzaji5T/9AXapm6FqNl9BoWgiMmoSPtm8BZFgCFFFRpA2L103xxICCTcKUTpWy6p6m5UdmSQhU65iIEdSR4ed96I3/4iqriMYoDx0yHDpNSnieqUhQlK8prT3aiIuMc+f9/AMNxqNCqEk1YR1BZfd+Ai6shoss8yyXK+Oe1hLEK88eDlaJ30Ztiyjmi1wGsOkrquWMmxxrrXB/X9iuJ6he8fL8Pmtvz7mFHUHFc1EqVLm+tf6rbvQm69A9gVJzsIqHM5xVSFpZBgj0cUX5RQhxwJKxRK2bNkCx6jg2m+cjqu/PZNPwjPcIY9BjsuVmx2iYZZJ10nqIVa2uAbEb+hg9it/weN/fh533XcHjNgw2FSy4ryBlFyibkwPikZ0POSMtGoVT7/4KjbsLiLUkEQ0HkcoHkUoFB6MuMIjk6xTASlj6WvWzhJ5IQE+MtyZrWhqbER8wrHQ9QhWLF+MeXPfxd68ATuQYqOoUv1OE6TI+eecgW+ccQIKpSzLIelBx0JsOCl9mEF164tk6PRG9Ds6hXSuhFKxikymhP4BjevDp37xSPiUMhzbh3S6jIFsDh3tnejv70P7gQFkzDZEI3EMawghlYrA55PR2tKCiqni/cW96O7fCccwkAin4AuG4VcDzHIqfhlUDqRlLJd02DCRL27AQz8cj+mHUXpBjs67znSph67JrgM5TD/vGlimjWK+hNee+T0qxQFUqhbGTjsOXekqetJpLFm0GI119fCTcyZqjYVvQ/VMj3xhYyAipiYaUpAgdplUcgPFCkzHxsjmFN565bfQqkRaimqHZ+gkIS2XCoKpGvy5iHOsU2YbJ2XfwfmmZxQE+Wn/hUOkUVZgwkBH1wB+ePdsRnwCFVD1wWTE9Kurzsa3LzkewcYj4FRMvsYsgXRhMr2up0/mczvIWwwRg14Er/31obXbg3732aLHnb29Rezut3njFasV7GvvwNbdnZB8IRH1fKqraiHjpbrVkKqKYJuAKiKSbt68GVqpiIRcxtI5f+Z8YjDiuh5ILKJQYnkP78AlRXj0SqWKUHCoAE7L/OnmDdj+2R441QxajjyDYTY7VFcaR8ZApI4HgzivIK1y1wDuefSvCDc0ItXUiGA0zLU/IXEUOS0bK0dfCSrLBQnKCKilysAD5zWjrbUZ0XFHo1oNY/VHy/DevHnYla5CitTD0nQm2ei4CU20pSK49Yff4U0fDoawa+dOTJgwwd1gYv2IlffIBzoILoPQktimEMEwkqE6pMzFe8OgRg+dy0UiehuiZpnpQX9/Gc+9uQ29OQOmYXGEN9xIWjUIHSXQ17MTjlNAkIxXjUCrUp5HJQoiIKmgI0NS/SiV9uDF20/D+NFJ2E4RPjkoUiZeZ8GU0rGtWLMbX/nBr/jY8tk83n71JYwdfxiUUAP2dvShK92DXN8AlixchGQiCR81oxCooLV2RRdebuvVT739MFjjddFPX7aM/nyJhUGXnv8V3HzdRdCqGsKhgGhIcAk24lM0rcycRa3hivRMyA5rm14OsiMBqhmxEdcgCmoGlq3Zitsee4+5Gk4XmVC2+PfL/3Ijho2bBCXQBD2X5+OgaxIIR8RLu6UkjiT/pE8eMtxDj8OzGc5na0p23jlJBz563jF1DX35Cj7emUah6iCdyWL+ivUccYPRCBM0JLimjU1Cf853yB+RMscnch6XHUdXVxf6OjqhOCbef+5OJBNDxudBB2G4Q5GYWEQG0czqEsRwFVI1EZeEGUYpi83bd2Dz8vcx6ezLYHXUJFMAACAASURBVPBJUQRwSTJaJK/7ggorlMsYJgbyBfzi3mcRbx2OaF2Kz4maC7zcypPZ0XmyGGDw/BQu0RCsu/9rTRg9ciRCY46EpoU54r4/fz72EHwKJOAYJkxHZpaXan7JgIQ/zroVlmPAJ5G4YUhg4F0kigCs2GLn4fHzDovumRxwyJS5rUUoXQm9sEMhdyK6ZugfEWoWlW4klXQg/HeGabNm2zaqLM4nKSqRYNVSFoZEsLiC9EAOezu6kM0UOOqWKsQtqKhWC/jWKXG8P+99zDh6HGZMG80IhYT8JjU60DEDWPnxAZx79W0swunuzaC/vweFqo5cOodcMY2O9g6EQ1H85aWX0NjQCNU2IdN6knF45Tc6drd6QYdeK4Qg02NVFEHlos51XEcGXnriARw5vomjG9dwXcUUfSaexrJ0l032IrFbu/1vGq7fJ8qEkC2YtoSb73oKyzb3uVSpyzzDZqJxyTM/RPO00yHbPpQyGVfCiaGI6xmue9H/VcT9rwyXt8AhjQdS18fPObRYtOGrpo+VL5v3prFu2y7s39cH+AMIx2MsESTjJT0sRWF6iIglDI2pcdvi1/ls+6dQZRU/vexMXPJ1OinKlwnGDhmrp0cm+BFPJoSHYwvyNjA1wAgWTexFyqJlzJ07B5n2Tkw45Rw4VhimQmSGDcu9eBRlCS6JPFo0O1DB/me/fBRGOIamEcMQikcQcoUMg4ZDqQBLHsWmFBFRgiXb3NJ298xWjB09AuEx01GtBLB6xVLMmzcXOzMGrHAKEhFTJCYheK5pXPp56r5bQfXH715/G0cs4glCQT87wNbWZoxoSDDhNXrkKIwZ2YqoP8A1cDIM3ZLhc0j2Jwg6Ph9Sj7kX0HbIcAf7MYauO62fJNaktsBPZQvO+zjrcL04i23JH4jfkbabriWhDSLk6BpRC55qmUyO5fJZVKv9qGplDPQPoFx2cNzZX2NisrtvAPs7u1Es6yiVirh71p24+qrvQfUF8ecn/oTmVAphejOviUWRmARkVEHOyJXUkiKJzlE0CIhcmn6fq5jozeYhOwoWvfkEEhH6W2ouoDyf64lMDlCLH8Nk9yJSXsuojzMqcf619dta4sczEHLqvC9ISGRZOOfKXyNTFRGU9xqhMBs48eiRePRX30DzmJPZWZZzOf47Nno3paS9eBCa+Dz6mI/YhfPu9R00VBdJ/JPh9qx9zuFNQR+mwdEiW5Tw8ltLMHflTij+CKYeMRWf7t7JjCiRIvFEwu388fpYRZMAlQmohW/7th1wDBtNEQPzXvoDQyPR4TDkOTyIS9G2kM8jmUzyoVMOzZSW46CQLyIeF0JvWi5SAX3w/tuIROphGjpCreNgugw7HT/lJ/T+XnGcFo3E9ER0zfr9k+gqSmgaORzxVJKZcc9ZeGQURVeVWC3PcCUZlmTB7zi4a2YLRo9oRZSaDMoBrFy2CMuWLsG2vhLscB1V/hmmizyWmiscPP+72/nrS39yp7thCaEIpRZvGHdN6Ou2hA8NkoWpk4dh1cZdWLlhL8PJUDiCYCiISCSKRDSIQCCIRDyBpsYYhg1r4xbG1sYGpJJ13FssSSoz5HTuEtUy3dqhR76xQTuUR4quE2om4fXmHlEPFdB5O1AcarhQBGHIcJqgtIyqVmFij6A2VBO2IWNfVxe6+tP4aNUneO312bANDTffdBP6+3vx1OOPY1hTI/ykTnG9DfEGQn0lHlTjpPIdOW4my0g1xShMkIx9uQryFdGK+MmilyGZFShqDVJhMYWNfD7nGq0LlV3iiq6HMLyDO4J4b7lr5BkHrTedK4lhDEvGGd+dhXKV0Jd4DVuiNhsVd/zwbFx20ZkIN4yFSalShbgCWxBmruGSymwI9oqU8vOgb609H8QJHWLQ3jlI3Wufc1jVQUl9tYJqoYRyWYM/FMK2/Xk89dpyDBQM9pWkJgmwiCHMOk7aeNSWJgQMChe96U07O3tQGMjCp1pY8Oz9iEXpovs5EngH5RkuEyQ2XRyDI5JFulmfn3Nq5ni9xaJo4/jQ3bkX/fkydm9ajZYjzxyMtMK43UK3y1YK2EzG6+D1eQuxYOVOJFuaUNfUyAV20pF6UkfBIjtsuF7E5RYz2YbPtnDXzFa0NjcgNeE4VCp+LF0wHx9/vAbb+8qoqFGGoQTNqfZaJYG76eCZ+3/O8r6LfnzbIISSub9TkGEE8/lC2DaSYRWtsoEjp47Avo5+zFmynZ0T9YN6qICCKUUkyqGI9PM0s9Tw7UUpLyrQavgUkatFImE0NqQYriYScSSjIaTqUtxumYzFEIvFOHWIxeO8JtTU4VeE9JMdEkdwj+Bh+o6dA8H1bDqNluYWbPp0N554+jms3bAJDl1Ho4o7br8N27ZswquvvIyWBNXgqZ9Y1GoDPoEk+HjdmjStH7XwCQZYlCJFLyzQNZBHUTOYEP1o/vOQjLLYI16KQa2mBkX7koAKnsqo1nBrIm4tS1RruLSOdP7CoE109ORx/o1PcJ3eg/EWCBWpWP7cjzFuygxYviiMcoEbTTyZI+nl6UFk72AmSzmuLerTtQ/vfL2f/bcMd/+KPxEi4YdR1bFly3a8N28Bxo87DKPHjMawMRPw47teQqYE7vUkqSCdGBluMBxhY5aIbeacC5xzkLpp3/79fMA/Ou9YXHX5RXxBFDrhWqxu2kxsMJqxLCa+iBn2hyJQqNRUU+fyOEASDGzctAlrly3BUedezJMRmMgRtQpeOIKqBJmZpLIZ2GAgncGvH/pPxBobkWhqYQEGl7gIiioSZJUWlcK38PIcDchIZBM+W8JdRE61tSA1fgZKZRnL3p+LVavXYvuABiuU4IkOTAgZhhg4YFl4bNYtUEwDt9z3Z/RkM5AUHxziCwjNUsC1BFtvwIRP0jCtPogjp4xGb7aC5978EJIpwxcQm5PzYArBlN9S1CASjjeX2OS80VwJn5fzeaQdfab+Vc6YiQ+QHS7JGIZGrS01yjgfrx0Zu991xuxguEtM9GgHaQiBP4D6ZB3O+9oX8bVzzuXOrY/WbMQtd97HnUiU85KTvv7a72HHp9vw1uzZaEs1MO/Bx2I7/Pqe06RrRpvZg5W1ZKYjK9AtG129GU47Rgxvxtt/+Q0qJSAW9rP80/V+zN6S4bLc09Wcc7p1SOViMBi4TfC1RkTOgpvyGShLeOHV9/Gn11cy289+jI6VCSwdq1/5ORomnspcTyWbHyTwWPOgqLy3KXhw6Yd18Ac3FXhOdojfGGLHBc8zdGR8LWt+IA1seM5hNlbXUcxX8MxTL6OxoRnDRo/EmLZhqGuIY9GmDtz3xDuQFIJGAi4TbCZZoUyazlCAWUm6EMzYOQ727t3LTm101MHsJ+8REccRF0hAWfrWRrlY4uhBzoCen8lkEIklEIxEWEzheUPKYfkhAYvnz0NfxwFMOfVcFCkMeVDfERCRPjzDJa9Ji05tgNf/8hFE6pvQMKwN4UgMikr5uegM8vJIoVl2F4zgNxmu5eCu81oxavQIxMYdDa2iYvG8d/HhilXY3l+BE61zZXyUU5vCcG0Hs356FUa3NOOPL8/BstWrYMsqVEtlgo9guUGmJ6vQTAthWcdRDXFMmDiCHeRDz/+Dtdgh0vZSzsk1bTFKiNIL2XZQJa0vORzSWrmdVmy07ugfzyD4Z27nDDszlrDSMAoS0IhrQamDQQKYwcYSV3BB6YtM4htBlDGh5xKTV1xyAa64+Js8fGDhh6sx68E/uq14JGJx8Iv/uBaLFy7C/LlzUReOIEC6c76MDqgRj5w+oQeueXKaReIGKsWJJhbarDROSTMsdPWmWc134vHT8dSD16NUMhBx94zYFg5LTNlQXMP1Jmx4hisMxW2i9wQbNVZL78f1cR5mQCN1HPz0zpexbEs7p5GDdWbLxtknjsHDv/wWkqNPZMKwSow3iXWIq3GlkGS4hMC8CHuIQGvwnQ8yyEMY5IOjMPE2LvLJbX2BySnabO+8+Q5UuQ51qTo0NNbDFwpg82cHcP8zc1G1FDhU5yRvTOof9kwRhBMxzsHIyOgARA0W6O7u5oVsifrw9K+u5KjI9UNipSUgGo3xpIlqucJCDhLMMyFB+YbqQyQaRyQWH4zQg4YLB8uWLMa6lcsx4+RTobSOdw2XAyRffJ6+4ZJUJPRnHbRZxX/85gk4RFANH44wvb9LFFHvKpdEXEb7nwzXBu76agtGjhmBxPhjoFf9WPju21i9ai229pdhBOJQJUIPYjIIQWXdsPGTb38dMyaPRyZbQUNTM9K9adh5TdSMKSKo1DoWgOyXIUdCiPooT7aglUrY2UNCBgtVU6AHypUo18vl85xH9/TleLJEe0+/iMLcpO2q0hiSDbW4MZrynCVbjnAAzE37RF02m80w++1FQYLBXjeKKgvikDckOW8yLknCz677ASaMaMPEw8finQUf4uGnX4SP5bEW/LKD6665DCsWLMHyZUsQ9QX4fD1HEXAFCpSymIYQt3qkIh2PcPBMx6GiG+jtz3EU+/bFM3HzNTNR1g0WdXgEHO2bcqkoXqPGcAUUo2d5wp/Pr9+y8R9quKaG83/0IPZnqCwn1pgexN4/8ZuLcNYpM6A2jGGZq1UlfbkhpJL0jrKCSrksGHhP5lgb2mu+/l8Zbn778w7pL++5/wW8/e4KDBsxAsNHDceo4cNxoLMf+3uK2NbeCVtW+KIodAFcrSoVmSPxGM9v8gfDorOGk3qHHUFPdzeSQQkfPHsPbMliVRItABmKbFqsaiKpXDAYQi6bY8KDapBkzOTZQ3XxQXKKYBLlN8Qi9nbux89vuRNnnDAV4864EIZFr0ksJHlKmwk2ryzkko28TE+/8Ddsas+jeVgbQvEEvx9BP4uQgNuT662ngDZMSPLgr/vPH4GRo4YhMeEYWEYY8956Ax+vXoGt3QbMcCM3mlN5SjZp7EwVti5h5qnH4vvnX4AVb6yAUwoCVZlzZtpcZCB0Tixo55IHnR8RQRThCOoR/Ddg+2zOP4WWmPo7FQSDVJ5z4A8HEIyFEUiFsD+Txe33PIS8prNEj6SlXFvnHI+rbKJBnZwas/Ui33JkEdm8/lJO9bnrRaAdzxnTurBTptKd4/Da3XHzDTj6iIkMHd+evwRP/OVVhtMUxJsSUXz11OlY+/HH2LB2PYJcTpShGzpHVR/X60UE95AaiVeYnPTQFaVQZABVA725PA8l/OOsn+L0Lxwp8uRAYIgDsSwUC0U3PxZSVeq59R4eKTXYDcQ0sxuBuaVU5J5iOJxIOyi9+MJl93KrKOfhruHSMS5+7mqMnzIDUrAeWqHE50TP4sDE7fsSpx2i1Hew0MJzEt7hfR6z/S9sfPDHUvXT55y5763Ev9/2AoupKUeh1q2pkw9HS0s90vkC1mzeD43ADeWDPClClDaUQICVSKQLDoQifNG8aXZ0pvv374Nk6Vjy1z8ipGgiMfdOQhKb1svHPAhAhMoQC1fjHW1R5qHSzorly3Hdzb/FT751Oo6d+R2Y/DomLEkIKMhw6XUJ/hNbyR0dkoRVn2zCy2+vQF1bC5INjbzIPJrHJ5RankzNg3MEKemYKZreM3MYWtqa0DjpOJhGBAvmvoOVHy7Fp/02KoEUyztpjpJtUS23jEkjm3HzpZdh3RvbAY2YclETpjYh0oYzqefIfHykt5Vk6h7REQ7T0DOFCTUOiyYpcUSDB8kYaepAMhV1yxIWSw2jagRGtIopZxyFWY8/g4+27WSBfG03CoEKWj/elK7x0eant6G1EnBSEEJ8XWzRTMAbj8tFYs8QLPSuz32/+jnK2T5MnTIZr89diL+/+wEjCVru8SNacfnXT8Pzz7yET7dtd6cdSowcOGq5wgpKkYiNp23BbLw0NErHF6TyGJAt0IA9mthoYuHrT6AhKdrtvPRGnJOFQp5KQaJ0WGu43kA4z0AEXBaKO36+a7i0CNFIlH9GFQq6Zid88ze8LqTY8gw97lex5C8/Qtv40+D4fKikxXyp2mkX5JQ5fXHX1tM+1BqpZ7i15NihxNW/MmBp2Su3OFde9yDyGimEZCYe2lobcMrRk3iwmq364QvH8dr7a9BbKHGbmOclZV+Ap0n4AoIkYMKHciDyzI6Dgf5+lkGed8LhuO36K+AjscQgoyY2iPA+okDueSLvYD3HK57nMXE22tv34BvfvAbTx7Xhmlt+BZ17dkm44P6lI+qAJOwW8Fv0QqYzRcx69BWE6+rRNLyNaXuewkc1atfzC9gp4JXQVVPwMznitrQ2oXHKcTC1MFYuXYxFC+ZhR7+Dii/J4nMGfJaEEfUR3Pbti/HRq7tgFkUOGQj6xEhP+nAlo0Q8eudNAwQo76Q6L11sPmYaWkDjarlPlyZOAtEYjZMFR1yCspSn+ijXI8Y1KWPy2VPx7VvvwYBG8sCh+UbE6guyina5KMsI4cOQ4MTLY4XAwpW2shELldbQtRLr/PA9v0ZDjByNjRf+/hYWrFrLLXqaZmHG1HE4dnwTZv99Dtr3HWBDpbDvGS5BbZYzqpRiiYkSwjG7cJRQCKES20auUEKupENyNHyy6BVItu6W1Ya2NeWTNCBOMLT/O8Ol4yFy1TPcVWs34fr732HeghpYvP35hSOH47l7L0F8xKlcS9bpfWlAn6dFIHmrSeo1IumGorln+IP72/3if2W4k+plJ1bXgC9+4Rg4RgnTp00k14yq6SBXtWlOAwb6s+guaDyKdOeefWxwXLLx+ZmcolojDdCicgIzj/4Q1wdtW0NfewciUgVvPv8gE0FM8HMvgVvXPUQV4m0e3l9eXZFgGsE+0gvQTCgHWLhkCSKxJvitPIxYC0945KYFd6Eo36CckDuEXM9Hxv+TXzwEX2Mbho8YjmA4yOdBPoGIEq/vWLDUohyiSQ58hom7LzoMI5rqUTftJOiVANZ+9BEWzn8T2/pMlH0pvgQ0toZkfU/+8iZ8/NxWaBoxzIQ0bC6zcOSndjIvV/IJFpfbJCUbdXV17pwkMQ1C6GIN1j+LlkMH8XgMlk11VAWBEMEym6NDPBbj802NjmDBgd14fv57sG0xVpSWmssr7tpQV5qAx+I9BvNaYtTd60ENDExCsx5UuDF+rivYp/N9+sFZcHSaNAG8+tpbkEJ+TrF6OjswvDGJpvoEfn//b5FnKEkbW+FZw/Q63JVFY13IoN3ha8KovZxQ1JlpDwxkcihrxIWo+Gj+02wQYkqlkImSsWpahT9c6onhA0NlrwTEsF8Qp0OBwav1iqBAxBR1X9GDHP3jL76J1xbsQKFcAKwAbNlkNv61h67FscdMgD85Fk5Fh6bTNXZ4TJD30Fwya8i1eNLcg37C3zDicaW7tbCaf1ejiqwNbtKcP1ztkGiaCu0GVNauHujoga7ZKJky9nb2oaw7rKSq2DTWRjBn9EGGq6gBxIJ+qEEFpxw1FVde+k2ESSjg2AhbNBhbiMp9chWmFOA+U8mnwMewzGVwCeKSQoa6gOhCuJGBUz3RwgKLSjMUIcgzWxYWLFqAYWOmYNeH8zDsuLOhSTSYusYDmyayuRzDZc9Tkme/7Z4nUA7GMWLkaFAHCJezaLIjf/YQgDsilORq1MZoO7j3orFoa0iiftoXYBphrF25EgveewObe6ooqUneQCSPu/obZyHVIyP7qYlSucqCAsMUxkuOiyINPTjHNbwoJiEeCXInlBeNvc1D5JpHuCXjMU4JyJ0GAz6efEnMeLVSQoqN3kSmUsLEfzsa377pTuhOCTppi60AoBK7Keqi7nivwfzVy8Pcyq1YRMo/XRGBt6qsK3bHzNC1ePHRB2BrJRSLZWzftBWG5GDNqtVYvGQRfnv3HQgHZNx5xywUCmVGNz6/yoorehApRVM0BFkl1EZUyqFUyHuwZlxR0dPXD003MWXiSLz69F3Mi4TDBGlpWJs324wcgilKYm4XEIsuXMOlTb9h/TpMm3bEQWUVNg4XzRGxJMnuPClbwm33PI61e3X0pwfAzs6h62di9as3oXX8VEi+ZlRI8OEesme4jPZchOIZJn3mFKTWbt0KL5eL3K//leHWlvj4er36++87FhtjgJVi5Dn27e6AIUnoyVXQmymhL51Dpmqhq68Cw5U4EsQhsqohGcEDt/07Jg9vwd63lwArt8Ha1wt/XueezwANOKeD9lE+R80lshj9SkO8KJ+iIrwfMGmjBP2QkwnIflUoelQHKs2Goo9kDJFTj4D/xEkw+srYsHktwnWjsP69VzDpnEsZFnq5G60NeW+PiRWmT9vDwux5q/Hemk1oGzGKFUgEjRSfYDC9uVre2tJikkMIeIbbmELd1BNg6mFs/PhjLHhvDnamHfRVfUKcDgOP3HwjPvnLVlRKVGKzWMNt2SROFwNzPWUWXUSv3jxy5EhUCrlBgTvls94xm6YYek5N/HpViOdlVTjPaJTywypSdcnBUgV1Ek09ZxLmrpiD9dv3Y8n2PiarPJKJ2dqaAfRetBUbuGYSBXEQg/ppsSJkFKyTdpveX/rjA7D1Mk+szAwMoKOrk88zFg6jpS4KSyvil7fP4rtJ0GtRbu85K1p3ym+pU4rgMR0Hiyeo1cF1oMQ/6DbQl0nD0B185/Kv4hfXfpMHG0YOMdx8ITvUEfQvDJfSD683t9Z+PMOlVk8aLEc5r20pePiZv2Lemg4eAqFTSc5S0NIUxBtPXoPh40+GLIdRztH7esMlxFBFRnsui+8FDe/9/p8Z7uyHrnXIQ9BG4EWVVOzZdwCmRcJuDbmygWLFRJpu79GZRbEsBpEFVBUTxw7HCw/fgX1Pv4ny3xahmVhTy4JORjkIwQTsYxKopuOfvCNdZN44rs5YnKSASsK7C29Kt5fgMpSiwnfTv+HTrn6EfQ4yMw5D+7r1GDZlBhNUVCIgppE2vUZif53GwIioxqUMy0KuVMHb7y+FJgW4XzUQDKNAYgYSRih+FsE7sg+qTBuUDIhezcZvvzkWTfVRNE05EbZUh/WrV2DJe+8gmQihLpnk3tipRx2PHSvzyO2qwqLSEOU5VCs1RR5JkNbP6guX3TVNtLQ0CSTh2Oxo+JYo7JldNVu5xHJH2uRapcxaZuqljYSo3kjGX0HbyGZRBnFhV3B4ECt2LcTuvQfwzpo96Ncs+AjNhEOIRxJC8caQkGCP28pI8kFXqebVK72OILIjFnCwkIPKLQ6CqowXH3mAO2b6+vtQyOYRjkaQyWZQLlcxpq0J+YF2/OK2X0ORKbISchDQnPy2SlDf7+e/p3Wn1ITOn3N5cuZUEqJJoLaEvv40qo6DR2b9BF8+7Rh2eMGggMrMHtLAwkKW0wbBJAvz8FhxL+p58s9ao6WrSyiSrg8TU44Kw67wbO47H/or2vsr2LW/B5aj8nD1S75yLG7/0SmoG3MG5+Ua1W9twfyzU3RJtiFmXPSY/1cPdqo1TvJfTcPwXoMj7mtkuG4uyPS17EOpoqE/W4AkB1Ck5vqSxl0fNB7m48274TgBtKYCeOflx7Duhvswav2AgIPEvhEb546uZKke3cbD1aSqzpDQgVQ7NNWQ8z2X5fS8E0FKEmnwybh9v2yQkoRqQxSNc+7GppN/BPX2i4Axw5Hfvxtm8yguVYjiuchnaCN4zdqstWV9LDD71ddw5umn8t0HaPRJKOjjMo1m0R0GDOzsSGPSxAmY++EaaHKUZr3jwUsnobkuiuYpJ8FEEhvWrMSKRfMR9pNEzo94LIkTjzsHi17cDVu3eRC7ZwB0dwOumxKB4U7tp6maw0eMEPCONrM7eYGcZ5SYZWKp3aFq3NRNqYJOUjtKFQzWLVO0bWigCRWWmG9EghFqUE/5YLSZWL1yKd5euA4b9w3wZPdwUMW3vnwKlrz7Ks784pfwyYEBZKsO9FAYCo0gqelh5fUSN1Pi82eGlCWJVHqTEPH78Owf7uc17unpYeecLxTQ1d2Nhx55BM/+6VHk+vbhF7feCdumqZQElwNsUrTfAm5XD527lyKwcMaVzYpyM017BPr6M5xivf7sA5h8+HCXlRe3BiGWm4cdVopC6+TCYxaqHHrLm8EykyjveA9voiRBd3pNmvl1oL0X9z35Jj7d14dcmaoT1J0r49kHvoPTTjwCgYYpMGhyC6Eq13Dp9Qi91g49F4TgP5eDatllrmbUPudz8tpDI7f0/KzLxSBb1iJTKUblG2gRPCYIoWkmjwwp6TqyeQ37enqQyxmY/dxDwOLVCPz5A5gEAWkEDTUp0NhN13N7hjsoYXNv6ET9jjwS1VXI0KoMlYAczjW5W4T6GrmGKYkB5pA5V4r+6UbseOlNZHr7EPjFldi//D00nXAW3yFALIjDBundqMzzvASVaNPdcsvPccIJx2PSpMPF/Ct/kEtgsWgQYWJ/HQV2tYiySZMdbGanT5/Wgrpk3DXcBDas+Qhrli/CivXb4Jg6vnPxZbD3R5DeJ6Zc8M3PPPUPRXSXLaVxK4Q+6urrheCdWt34njlDk0VMQ0MoFEChkEddHT1PRBVTozUTs7CIzIKkI5GMIOgXih+WDdo+FJw8Wk9qwfxF89DbX8Vjf5mHlrY6nHPSDMx56SWG64c3xlDvDyHZ1gC1uQmfFVR8mqEZxUIn7m0URkS0nu45UeHMr0i47gdX47ipdFcGEz09vdi1ZzdHm/vuvZcVXS8/+yTSvfvwy9tmQYy1IqcllHVkoH6/mJfNyIxHBymMSLgk5DLZPAbVtJGjMo9s4aN5LyEcIsmoGBzvGS7fQ6laEvk3BQ33TgS1UY73xb8wXO6G4vsECRRChjd37hK8OG8j9nVmeFwxlaLojhMfzv4ZRh52JJxQGyoDNClTnINXU6Zq7v8Xw33lge+x4Yq8hXprxaym3nQO5SqVJGQUylWkswXIaoA1t+OGjcANV16GjsvvR7RiQyGFC3kaunuBIyLloMzLrft5bCVtANq4NLOYWU0yWpe1pIgkanOiBhbwk5TSHSlDdxzg+wYpSI9MYuLDt2Ddt29F7398Ax2fzMek2LoysAAAIABJREFUf7uKo43nyUhKRyIQik7UIUQRi2vQEnDnXb9DV15HXVMTR8CGRAz18SCSYYVvp0JN33UN9UiFowjTqBufgekTGpGIh9B8xMmw7QQ2rluDNSsXY9G6nShYPjzz61ux7m/dKBXLyJDTc7tQ2Ou7JVkel2LbSKXqWHBBtURyWNyd5IjeUxHZ6H44VdTVpcRgM3dig2hXFvmqblSQSoTgUwzWM5N6jYYDyLaN3lIZU86fgtmvv4RSuYx0sYot6z/D5s072KHQrVbaImGMTcV4cuaxXzoV7819F62NIxBuGY0NPT1or1AUUOD4ZKh0fUg3yt1TfvzsB5cj6VMwceokVj319vUxYqVzpTbNx558Cj+/+QYM9O3HnXfcC10n0YmQ/nksNZ83OW5XhEIbn/6eBBqeSILSpnK1yudAfMmmxX/lu2IQt1JL4hBTTQ0G5JQFiVMjruD+X1doUSv+rY24js2pCDsPEn0YOq6//XGs20OTN0WLKBXkaDTQ/Jd+hpbDz2SupjxAY3CH6rfEy/C0i0Nu3FVLDR+EAtzIKhx3zQG5XWMC4g9pGWoHWEh/++1VDrfEmeT5qa7mZ8Pt6s1y5KAhbDQXuT+b45IPlQN+c/vt2HjHn9DywU6YpHnlOaokCxNpB99gxKt7eY3i3GcpciVSp4joKHILL+IO1hm5Id5AmObluvI3rrdS2YRQgQ00Ln4YC069CvPVAdjTG3Hh1TdCc6EdvTcZiSB/dJEHsXqI2GMHn2zYiuf/PhfR+ibEUg2CuabJiQrBOIdvSiXRBShloCgmjhnbgu9fdBbqUjE0H3ESbDuJjevXYM2Kxfh0XzdOO/NsNJfqkN6pIJ8roFwSrX2skHLvS8T5tmEgHokxk025aTIZ5+dwq5/bZsdyTa2M+oY6Lp2EgwICewIVT95I+W00TPet0aD6RcSgzRcJBtGRLmL6t6bjuRcfxrixI3HLLb+FZft5YgjladFQGHU+H844+WjUtdRjf1c7OnbvQ8L2s6abjC+YiOPEiy7Gg6/MQzAURdhvY1RbIy788uloqY9C8ScwbORoXlO63SfZBMP8aASf7dzNDrF/oBsPP/QIHJvu9Eh3InRvRObuUS+F4uvqTj6hurSQPorNpBni9qWQqti46G9s2AG/qLXSg9YhmyVmlyg3t7zDrYuuJfDGHyrBHZpriroveE9yDm8RJ2Pi4usfxq7OLAcOErLQq/3HFWfh6kvP4NuMUJ+uWaSJk2Ltee9SfuuKfw5ihz8naWUU+N8w3EHKuqb1mt/v5fu+6/BoSy5TUKRUeeGyuQqqVBCn4rthIpMvolQ1MXnSWJzzxTORu+Be+Gn2DhkJyfP4s3gb2k6DD8/w3FGuRDTxIGxvzpNruLzQrsaWNi+RNNQB4w2sE2NT6bYaVHpSoc76Hna/+yFy23aj9ZEfYv3WPWgdNmJwSh95cjYe8uDuhAUSB5BEngaSjB03fLB5W6ObSeUK6M6W0NWdRldfBnu7+pGvVvkeMOefNAbnHjMKsViYDde04ti2eT1Wf7gIAUfCzAvOx5IX9kIrUBsXOQshuqCITw/asMSYUjtkJBgWEZSaHywDca59i6Mi50kbNx4VZZ5KpczrRPCVmFeqkVPkoteiOzqQzFNyKpAUMaKUcmES3g+UTEyaOQVXXn0F7rj1CqSifnSmy5g7bzXmv7+SeYgff/+7aO/eyY6G4N7WjVuRCIYRsiU0NTdg5NGHY/WWTxGoH43DRzYhEbIQRBWth02H7I/yPXubxxzG150MlwYIUB6bzmQwefIkrF+/ETt3bscbc+YMGi6thefQyWF7hjuIOujKMMnmZm+OhAoNNzctHHf8EXjmtz/jyZWkba9FdMQXsO/9XxouGSbde5mOg27fSRNGv/6jPyBfpuFwpA2gY7Uw+/fX4Jijj0CgfiLKxPBXqTQ3ZLgUlYX665Ce2/+HhkuWRXeZlF598FpupKc3oy4M2lQ0y4dCfpXuuseEEzGeOuh2nHfedgc+/vHvkPz4AE8CIHtj76HSd7X26pIbjsxMH32QekbIzWjciuhYGRwOxtIzMUCO2GfOrWoWgEem0hj0ACm5AnDO/wKkyeOw91ePY/z8h7Fk3SdIJhvEAdAxU47Jt9uk+7WIIWRC8yGc1D333I+jjp6Ok086Hg11CTTWJ1FXnxDsNwlFJBkawSTLwc6dW9EYqqIhlUDLEV+Aoddh+9Z1WL1yPoaNHoV4cSz6t1aRzZdFlGe45E53cNMB8mU08pNgqjhEGv0pBAGJRIJvjE2GTvXkFN2ylG+aJoyUYCRFFoL65XKBG0AYurqN5o5ThuqTEI8HEY0m0ZfRMe3iqbjm2h/jsDFNOPfLJ6AhKSPATRVRZLJVbNu6DTv3tKOvP8tD4j7dvoenbM78ytlwAg727tmBq666ENt2tKOkUeuljVR9MyLJVoTCCVSrJkYfPpmhPbVxljWhWuKvCwUcaN+PbZs2Ycvm7dCp0lDVuT3PKyV58lIBB4dKTN6m9/gBru3aDh741TU490snoFrSWdsucnBxl4F8IS+kmO72qyV+vNzW4z4+rxxE+zYaoRo5NTU4mLt4DX7z6LvMNg8y7ABWvfwTjJh8HORwI0okc3Tfj3TbTGqR2o3aVGv6bcV+d8VGh7TmHSSo+JyWv1qozOvi1oJFxL33KjEBgzYKTwChhmQaOGawbEvcmYzIFgmJRArf/NJMtF94F2waRVozlsNWRH7JCh0XpQjqX4Wf5zKTzlnh16U3pp5Nd6KS2MjEDjJcF1MXPCUJRyx3tArDKVlCOBZGaVwbmm7/HrZf9ksc9tjN2Ez3EyIn4d48igdeGyaKxQJveu735fooMc90v9ddKJbL2L51G49E0S3SvgYgwxT3DQqqmDZlIk6ZNh5/fOJpzLrpSjQ3pDBs+inQ9Th2bN2MtauX4vwLv4Flz+xFrreEStXkcyAvLfS34jYbDPdpNCmL4l1JHzU4KIpotKZzClJUtZBKxQdrpXSlquREDZ2b3akcFKF7tsrkBN2eYZ6aaBAlgngyiFisDgMZE0dcPBnfvfpqKJKFyy69iG9mXd8Q5FG4VIMncQSlPnmN7ujXiAULluGEk0/Axg2foLuvG3FVxxdPGEN3H8KBjjzau/qRaBwPNZhAQ0MzO+ymEaPYwZKx0qhUijYEZTPpAaxe8xHynb3YuHkr3+FBqw6Vg7xI6+X0XsSla13bm0vPo3SBHvNeewwtjUGYBh2vN2mSFFNVvpuBUOQdXCUV9wcWZsOTNEXB7J8EGCStJGfgkYWPvfgPvPTOBkZF3iMOA0te+wnaJn0JUMIopbOD+mRvj5Y1ocOujbiC63DFF4ccn2e4h+qTa2G21wLLebB7D2H++qW7r+S2Pmb73JDJ0xFNaimjmh01lBNDClxwwYXofOQt1C38DDrlIq5HooM16Z633niaGsMllVmMJt7R0bu1XVG3GpoEIFg4TzNLKllvSBqJ/N082O2fpIhLA7H1VAL1L9+ODedcj8SFZ0O+9DR0D4hiOF0fJr54lAz1xgqxN9s0T3OUEY/IaGtOusSYmJ5Bf5PJVZDO5LFp41b059I4bGQb/vzim3j+nmvQ3JBE27STYZhx7NiyFeEAsGdNHunPLKRzFaJAxYA6Zkf/D2vvAaZpWV6Pn6/X6X1mK2xhC8tSpCpNECkaRIiKKGpECEaTGFvswW6MiUaNvUTUGA3EgoogVXqRXVjY3ndnd/p8vb+/65z7eWaHDf5y/f/X7/PyYnd25pvvfd/nee77Pvc5567Okfp1QoZpZ2uSNz4Bps8Uk3MkChcf9aukLcqczpcRJC0Qqa+yHdFET5eZk0s2x7GjAmPYTuFxVEY6E0Z7Wx+mcy2sfc0qvOb1b0YrKOOyV1yGJYsXorMtivZsm2h7nekU0tl2RJKdQDiLeqiGZtWECZzAMDP6LKKFHRrSzLGos9UwxvPtGtZGVgkdL3sXLlHGwJqYLUQvp8zlpnHfA/cht/sANu/cgUKDtEBGbYciO902Nyb/L2TZtQx9EOF7Mf1n+s1rvP+2byOTpjcV+eVHjMHp4czD4k9tXLYIvcPin9q4HOotzrTQ8xre8nf/iKf3GxjnX9dceDw+9u7LkV50EoJGHNVC0Y1PcYMD6EzqpkL8v9y4mmPsAUy3cXXYf++mNyriCjmjEXeViCbnzhjTh1pWCr4TkTje+JprsO3PbkK8bJpXOdITTSYSKmd892JYd9pY/lwqEhNYpAfFDyHp3xEfKv4b00Iflf2pK8DfnTSKlVqknMERRSQbw/BvPo/Hzn87mh0pLP3Jx/HQkxvQ1dNv6bDT5Jar3LhszPOhW7pNjPCpDU/h/ocfxdmnrsXKFcegr7sDwwP9yKSSqFFTWq1g4zNbUC7PYt3q1Qg18+jMJDCy9iw0Wl04sHcvGjPAhtv2oVys2jDtqi1e/g4PRrGu5QHCF+VgbOewbJBDZjyqw6RULmHB8JD8kxlRBfTxMGUJ0mxq8bLO7ci2SeqXTFEfax4NYn9HCMxwpEkL3b19mKrVsOrCU3D1tdci3hHBxZdcgHQ8joHBfoyMDGrIeCKRFuHC6249+OWf/9jOBxCrjavGIb2QQpJqPYotB1tohNpxzHHLNN6kt7dfzp78OZFMmk3kCtMoju/ELT/7DfaMTgrc1CesmyeTRSXvV2aHz/ya1QcSUmp17dEQ7vvVv2jTUoTBA8Be5jEldJ4JqaslSRDxLUBRIqVNdlxheWs9v6+aITDFz84MslHD+W+8CYVGCKEmJ/MZ+v/Aj96PJccMItK1As2CaaT5rlEHlHnRvI+4z4/99mntoLXfPT+d9z8zF63n/bA3kfNtOZJTcrOzCH3rI1dr45oEyfSbQv9cjUV9bDVo4lWvuAKJ+3eg8tXfolzhsOqWLFcIHinyOlsSF/BslksohAy9mWnpwtS4BbFlJMTWyA9nq8oeYcvpK90GF6+TrQJ/ErOdIB1wBIloEvG2BAZ+83ncdcENiNbqOOHBr+MXv74DI4sWO8M/A6c0woMR3cnnWAs+/dSTeHb7dmzYM4njj1uJbCqJamEaq5cMYO2Kxdg4VsepKwdQZe3UKGKyGGDl0gH0ZuNYuO5MlMpJjO+dwYENeezeMIoarVnrAaanJ+eQZInznVuFZ+yQaMD0K0GATTrcCBrNGrq6utTKKJeL6t+ypBDKzxS/0cTM9AxGFow4ZRFRaLPaoVuj2mkRWoXS2qaB3v4+NDmlYVEPPvrJT2Dk2AGcfuaLsHb1Wov4PDCj1NqagyafA58/a+tcLq9NRET/0NbfIlKn/WkYyWQW1GLICxsxHJyOonvxaeju61Imtn379rk+KNfR4Z2PoDM+gV0Hm/i3798ubWpUm9D0snq2nPLoDmXeE3HfSXF06LsypGhcAN2CgR784gc3CYPpbOtA1fX9mYTRUZIZCEOB5y2bx7IbSSLFljNadwHK00l9nCFH2Ud6thbOvOp9qJEp1YqK/94KSnjsJ+/HwjUnI5TsQok+TgoqvOfmeOqHVv/fNq5tWPutz0Odj/r70a0h/71+MAFLE23cud5SyBrkmprt5nmSh3rM4mNwxZVXYfMVNyFxMI9yhDR3jdIzxY53p3cnmZQ1gdmhhOsEYQIEZAxxwyLkRNQEpqxtxF6ZqXNss1oqaVHba0G5+Yg0c1GlYmkk2xPo/eVn8ftXvxvZyRyO/f4HsTcGlDkpQJC86TvpFkG1E69ndO927N+9C3fe9RDOOvN0TWmgFLGcJjlhDdKNaTQD0h3LSKbiKFcpK2vg0FQZq5f0oTsTxcDKU/DcxlkUt7eQH6/g8MEpcGod20iVWlHSMtb+vB7W5MpmXJSx4VQ0SuNwZx5CQAeBKKlDGGHJ260jJZaYWfLQRYGqIbUbdMDVEI4Ekglq0gLR5gR7rsyLqiDvOdTfiX2FGRSbdSxdvQixBEn8hkgbG8oOQLHaHNWO6b1F2zqmp6dQ3H8vx32pHKBgX44VkhE20azk0X7shagkB+R8snXrVr0v21FMmw/veACHJ2Zw2gWvwdo1qzA4vEBYSaRhJRmvSxFOuAPlfkckfWSzsa7l8+PUP94bfvZjFmVRJZ+8JQs/A/doMkh2XIuHc1VMOO7XeqWEajGvsqXZpJj9+fFPQWWeoES2SS7D2bx9N66/6WaUajzsSSwKY2Aggd999Xr0rXopmmHSHE24ImN4d//oejL/PV8o4v6/2Li8Z3KO/M7HrtHG1eZl6sshRw1LPfggOX/0pLUnYnVyBOUP3IwCpVPhEKpEbclJ5hnujjAPIvHWZhNJoau68X6AsenEjEUTtsl4Qu2YsGmh+ka5a09pELmrizgtLm5NegNzsuj+wXtx/zv+CalDU0i94XzEr3gJDu4dg1YbT0oynypFjO7biX079+LB+x/FqaefiGUjWVSaKUw1ouiMtHDuRWcgGy9jyzM7EImnFfXa0hFUa0ChWcIdm7vwjj8/C0G1iR2PHEZ9KoI8J9FXgWKpigpBiQCoFHJz4BRjgJElzMmCC1GqKkaXaEz96I62jO6B0HUnvZODR7lk8j2SUFJ0Z3JSSNrjCHmvIx0nfZAHBAkSvCf8piqGhxei54xj8ehdz6J/ZSfifWkkmeqKceVSSPc8dLAgsFm3bEXVyzg0MYG9G+9DWyyHRCyJRNJ46VznTOtJ8avUm+heeQFqsS75aG3e+Chy4/tQL09r0PSrX38jhkaOweiuWVSmSqiXWwgaYSTCSQcSATVmbeQ/Wx9HBxEPEpZcYs0xatJ1UzOrbAazZYYE/VxfWzArwTb+n7RrJ1GMRhBLcqRpCBEePHTWFFehhuLMKAq5GTRKBi6RgJXiemlGNIPqi9/5OW69Z7MkmUrqQ3Vc/bK1+Id3X4u2hSehUamgXLaNKwsn53c2f+OKduvCuaXE89qj7utHR1wf/Y+Oxv77+F+uHw6RV6bCGtejwwTD6bzATgM3pdDRRh03/PW7cfDyT6I8OmGm300OZnD6xjDlbNbw9myYGNs54pG63N6hajYo2kHjpInF4oqOCTGirKbWAcKmN6ODU13we+gvNIe+hUNoT7Uh8aXr8dQX/gPRzXvRXLcIa778Hjzw8BPIUGGEFg7v24Otz23CHb/9LS6+5CL0t8WRbx8GFq3D7c8extKggPddPIxYiDV2BZs27UGUJIZ0CskUS4YYRpaegFhyKWrUunYPIRxJINQyMrwUILocuyamv6qtXKtCaKZzYWRWIeaXAqlzkaCG2PppcyNLXTFk0yO4aOmNWaphfHQc+zbsxaFdh5CtAbVWHQnqiNlWUx+9iXC0jmUnnoCR01fhrp88hMWn9KOSILMqjUajMufQQNM1LgJ+1q7OTul9efJs27oZDzzwAFr5fThlzSJZtCayUSREkifzDPLLLlXr6Ft9EZqJbokAHrn/12gWD0jBc/3ffBj7dszi0MYZhMoxmbrFIgnEogm0Yuxx2qTCZp0m61XDNgIudIIwIsJqHXBTZ2iUJ+6xH89iYBEzKfWB4zHZBbFDwVKDmQxrYvbGs9k0SpWCEytwsmAOQbKEdGcYi45bjL5Fbdi+8THEawXEU3EBs8RrXnfjp7Fnqq55b7RbCocS+P7n3oALLngJQulhFKa54Q3V9mWcNyb0m2+OSDS3eY9syxfasEf3fefXv/77eRhQUTU+Pm4jbpkqe2dEblxGXDOlNqeGNWvWYH3bEoy/7WuohWtqEXF4JS+S6CKlefyzr5OZdoQbHIdxhMblp5dJRO6dLlwkFuLqmE1e6eE3rgqoUEh1sU/ptEVcxE1+8W3Y+NVbENm4E6GuLJbfchMeeuAJNMINHNy1HXfcdjtefNrJGBjuFEmkmBzCg6FVSCfDKI4fxKcv6EQiYY6J9InavWtSiHMknsWy1evQO7QS5UID44encHj3DMKtjJz0GXmYlgXse7vDlAswVDEBPr/Eg4douVwe7Bh1BAu2TCylo6GYvJeUOpo3NR9QNmNDuwXShKugq3UoHsbgwi4MrBxGOEjh6Z88hqlDo5oyoEjVaiLbHsPQCauAgSy23XMAx5zRi1y4hFYoiliUtaWz0E1nlG7RhJ7kiWwmo7bUX739HTjp1HUY7O3HxN6NOO+01UhlNULc/KF4knLj1uoYWncpCi2qfkJ45rHbUchN4Lrr34MdOw7gwKMB6rPMMmKIJzkegrUr3TzswOJC5zrh1AFNwZCYgCouIpos11rIZGn9a4wrDz4RByFZhPeUG5seZELwJcYgDbQmmihpsfVa1cayhO2ASkVjKNXKRvmkk2PvBE695HTM5HehNXtIffFys4lXXPtJ5Ko0g6dpQ0ssugf/691YfNwZCCIdyE9OIuxYXv9/Nu4LtYDmDvIXiMZz9S1bqAHU3hRH++sfulpjNj2STPiZtSajZritDW99/Zvx4OUfRv9YFWUO9Q0a0qgSU+OLaTLBKaKfYrQwySYfmYvQiQV4E3giakKd5CG2uAVUaSaa+RboQzohtUcWiTSL7ujkfiZcCCGRzKDna+/C/f/0HXRs2o9qGFj/u8/j0c3P4cdf/yZGFgxh7TFDWhCToTZsjS/BWGoY/ZkqTurKoK01g/VdeRndNcNRKW9K5SaaQRYrjj8NhXyAJ+7eiWY5jmSQRTJK07KyIoD/TLwU7+Mk0MWl+joI2f4IkRTRpl6sH0rFQ0pqGA0Kt4jryfY8LAlUkQ7Jr6kH7HqWjteGYpBDrDOMky9ah5n903jqJ3cp6nJywPpzTkPn8Utx/2+eQKsUQd/6djRTVHwRjmiJWcWDktzzvr5+/W4DxUr45Kc+IVLGmtXHY8XKFRgcHMTeHRtw0vJ2tCeJS8RkYkcTOtIQB9ZehUaUHtoFbHnyTrz4nAvR33ssHrh1G0JFNwhOPttpM4j39rFaNJR5RrV5D48ddqbvtBsS4VkHisz+3ARGmRQ4RhXvC1NUlnEkPtAhRL5ijYZkebzn5KdzQ+vQ9JMfKQ/NsvVWNgAwEUE9lsOLXnk8xkafQZ3jQWeKeNkNXxDhwzyom+iORXDHTz6AoZXniAtQIoAXCsReYp7N0sZrjL0HwP9oBx0ln1fsOYqk8UKRmBuVpRS/l8+N4KE32At9+X1XBfkCJVGqpFwqA4TjCbz+DdeidNcmFD/yY9RpoK1ZKnVUgiZqPI3omsHZn0ELiSgjp9ViVGjw3eYG/BJVZBokiVgY9UoVWfZ2XfQNmnWxlXSvnG8sN65O5mTK+nxOZmZ1CaV0WQz998dx719+Coldh+Vn9MiKOFrr+rBquButekH1y2TbSvyu0oMgkkF/OoorhktItKYxsmBYn5uACXW5zAZqzXYsWXkidm+ZwdaHJxEPEmKRifwgIoQNreZnNA0zU/2q3TkN3wqLqcVoy4g8ODik+lcnqrdYEXKcVirsWVSMsvTnGh4Z0kMi+urJCfwvFzEXinjg4SjqdeZGBay+cJmMCh7+7s/R1tWGkbPWItXXiQ2/26nIMnBSL0LtDVTqVZvQ4JhoKSmh2sxxolHRDCRGP1r5DAwMoVgsoVQsI9PZhf+6+WZc97oXY+FQCrGALpxllGsVLDj5GlSDMPYeOIzKxG688rLX4g8/34RosQtTM9OWlgvDOJJteDCK94MHGw8SbsDZHDnhZpFLbTP71myRzecyc+MKvHSjZmy9UOJY0+8hMkx3UOv/0kPM7GR9RFd0VvvGPLzYimPWkRho4awrTsOOZ36DbdsP4C8+/E2Hu9iOeN2lJ+Gjf/s6tC04AdViGZViSZx2yhI1b5FtR41OsbzghV5HGI82GfKFXkdvXMtgW4hHzR2T94Ke457aGvrSe66aG2wtIUsQYMGCBbjqytdg9y8fQuXzv0S4WBYPuchZIZzFE4ZQ5fkblxvS17UaHiKKoYnHaRKn9JLIKf1wqf+UCNqRwnVCBjYJ0NW53KyefM8Tle+p3J4pJ10gkiks/cO/4t4L34n2XFluE5lLlmPy5Da1UHhIFDIj2BJbiH2zUVRTKRzfHsKFg6PoiqYRontEKY96JIUo+UHNLBYvPwObN41j15MVxOnWWGPmEHIjNG3TKhJyKnqCdVtMOmSypJQ5hAJtVG7c4cEhM+d2TB2zPJUd4ZEeYxh6H24a1mVqkRklfq7eTyWSSmN57eZ6yHlABiiVG2WcdsUa/OG2u7F8aAiDJ6/AH371OIJiQkDMglM70cxQUxdIqmhtmADt2YxcHSbGJyQG2Llzp4gqmQytUt2w8loZPZ09+Mb3foBzzjoFs4f34KLzT0BAMghaGFl/NSrNAFt378FLT1+P3c/mMfF0AzFwYqD5dHNyIfvFVrMypbeFLvFFyAzQLdMiQ6wsVRb/3ffxGXG9nlrtaqeMkiFBzAQRsrVNJPRMiMlYKspWkrH1zB0zhnQ6g1yBEcs5PLoh6mwFHvfKxQjFpvDFL34B37rl0SMbNwC+/Ilr8KqLz0couxBT4xPKquZvXIFSDmT9U4L5uUkTDoQ8OuIeDUhpDbjsjbiJ16ITmCI+0NPTjdC//M3lQaVUAZdYR7oNl1x5Ffomm9j0jzcjtYXeUzU0WpYYS/3QMgd+3nKf/un0m0fnkku9NquG3ZieViMOzU+XD0fTRwlaOSKab0kxCul7mSI47ylRvTiPxonr+Tniqxah55sfwtbz3yn0mLDFeHcdnTecIiBmJ3pxqG05ikELhXoCK3szuGgxhxGTwUPheVS+WqEwD400+oaOl3vjY78aBWdV2pxdI6aoZcUSwpl4+2xCEYQaWDXjAY4rpTXr8PCw0nn6RstbqkHXCjOCZy+OAArbLpwLxDRWEr6uDkUfLbzA1CqKtGSJ1ex3mzyR2s8kIrR3pd9UuIizrj4VpYkxbNk0huJuShmt5ZJclkMrxjQ9QDbZgUjcrGjp7HF4bEKLvrszi/EDBzBLhU+oimxbO9raOtRZYLP/jxuewvihcaxYuRLReB0pjcoMsO6Cq9UJHCBIAAAgAElEQVQymZmewmknnIG7/v0pRBspgZoh9toTcYyPT6hdxA3EqMQD1RBiUwlxbXlQjwuSm4ByT4/K8qDXuhC4GTWXlgZlf+zvGwmDmYW8tJwzpt+4mk6hEbCGkZgtEbM4Z41LJls8pjWFTAtnXrMeZ7zkbOybkHjYDuJoDPd8751YftK5CIXimJmeNhFNxAziuUZZNhjZwzJB/3p+BHXdE/fPR9JkI58cDU7Nj8g+TZZE1Q20Y5kT+sxfXhqEolG8/GUXY0FXP7Z88gfIPnEAiLG9URJqR40tdYdawMT/ND7DFrTAJdUtR6RTcdbIRN48b5OFPp35aMjmUmEvPPDjNv2HZZ3X2dY+N3PFEnjrmc3d0FAU3R98ExpL+rHv+s8beMOJ6h1RhG5chkIrid80jkU51g+EGzilK44Ll9MKLySHBdY4HBAtCh5bK23HoqtrBX73H88g3ezQw+Tm8iNQdPKLJGCgiGbUOuN3Xg8JKeoNIkBfX49NDXRRmJvWxlJwIcXQ5JAzDTQzJ0GK5tnL9SMuuPDoDOIXhr/H7A8zmvO9bJxLSDY4QTSBkRd1ITWcxnP/vQNNKoYcQr/otFGEMtMAUmiGqkhEF+PAnho279yp6fW7dm1Dd3saixYtlJa6LUtKJQ/hMA6PHsbuXU+jWi5icjKHgYEBtHdmZLNZyE/jFdf8lVojy1Yci8d+uxWV3TGZqzPzSZEt1uLIy5yMGFiTGnvNi9RscBkPJj5XZmDcyOxZlwp5JNlXdb1e3Sj18zm3iOJ7+mZXnUtkTPU5D1jzFPRjVRtKhXmfaErnN69lR3Xpodkvnxu3GY7hhCuX4ovf+Ta+9u3vuh5zC7FGHU/c/gn0H3uuDO/JWOIr7twcuaY5YcOCjnWXj46e8xFiW7+OeDLPLfOFIq7/mth2kTDGxsYlmeTfOzs7ENp730+DdCaLrR/7LhKPbEfAcQrxGKLsJ7YaKIUDzX5Viurm0BKv4wf2PFOdmvOkSxoxxGkFvi/bbBmpgIQNN6uGIBYXszyC3Ga2E9R0uCKHa2atG6I9r5iPdLZj0Z1fxYOX/TXaxnKgElgT5RIxzFzei4cGT8CziVWoVetEvpCuTuLCkRZOXpxGF3unjiLHeB8JJ9C7aD0ev2MclYNEP81VkadxscjhXdY3thnABKNs4zI6yhSedjq0gG21xCUmMOLBJ14Pa15mJNzAFBkImJE1KRddWUZvZFzRelSCeicwn9u4jv5otkIhtLe1G72QJu41m3JYQA4X3XgB7v7GH/QZJUrnwh86jJ7hHrR1pBTBSRlsNCM4PHEQd999L/bu3YXwzKSM87bt34cgTAM3G6FB293ObAsz41MYXrhIRu2DA0Pyj56amsAp57wSmWQCQ0OL8Pt/30YTSW2uNGcAhSKqH3mdowcP6cASycH1bU27S+F7RAcRa1NGHn7G/OyMwCZ1J3g/2G5sNJFMWDuwWiObyyYYWDZk9Fu2lqjx1s+xBEnSe8zsivje9LYiqNTb06PNG43xWVuGw2fYd0oGQ6tH8PEPvFeHAUe9DA924UMffiO6+46XXJMHC78/6e6RDPfnlE1cVV4PfIR+8T9BJ2c4f9Sk+T/VJlJLMBwSHsHrZ7Yl7fDjb7ouaN2xUYN6a7WyNgwL+UqNIzUomaE3Ygi1SADKhllnJTvbEe7IIDLQhXR/N2Ld7Yj3dAmsaRJYODyB2uPbMPHYs8iQjsaUpUrChiBl45UKKWa/17ntuIgtNJoqHl27m+cTCSPWDKEWbtIJHCt+9yXsuv1BlP/lZ3pPotriWUeB8RdncNeZr8e2mTriLT6YCBqoacpBfnIUo1u2Ij27F6evW45Tl/Tj5DPPxvFLT8bjvxxVRKsVCTqZCwgXlmeqJOOM0uZIyDRQIzUpgo+GFTm4YJgGcwFp0gPvm4EGQq40zZ10zqgza+fw62RMvTljLFUE1nChOeWfO73JeGqoDibSq1Nehx9TXqbzYYQTCSw/rxfP/nE/GhOMygROmug8Lo+Jwqz6uByhOjDYi7vuvN/8nQHs3rMb9cIE+jvasW+sgqo2SgTFUlmeWSesGsHCRUMY6O038If65MIspmfyOO+yq7BwZBjbHx7FxA4rb1hrClGvtnRNqs3CIYwdHtN/6YU8xyHmMvfuIPPMAhltZ2dmnJrK0Gmqd/yMIf6X78FDQUZ8bnCZzdYN0CZdrY0B5YHBTUy9LjcpTfdsdpUNPVOZ4xVunU2cfc2peO97341GuagM6MY3nouVJ52JSKIbs9Mzc4eFNz7nNTbny/H0TNxIl3kg1PxRKKZ0cbFX5aOjP7qRKEfSZJskwetkn533ngc761tluRte8cYgTOJ2bxtiw4PILh5Ez4oliA/0IKDUjNGJ2A0RPBb21SKSDoXNlUuIFmuoT+UskhIFI2gz0I9IbwfC6QRq20ex7X3/itkNWxBiZCKn2QZEauNycr3YRWwhEYBxHj6+leRPoiDKTR7F4q++D5W+Lmy5+iNIShroke0AzWgNtXOX4K6zLkYykcGuXXsw1TmM3Ng4cvkKipNjQKWIanEGqWgYX3n3m3D6iSuw4fdTKB+MolTNIxqwjmqIoSKLnURC/UHR3yJEdFl32onPGoosJ95QooyVkknQBMTQSJ2UT5dS8+ustZjCsfZltO2l/pe0OWY3NTeaIx6VD5ZSMpdicuFx4xAp9TU3nRrIGKpV+VwiCHdWccqlL8J9P7wPcW3cFtqX7kI9xujSoUl3iXgffvGL2xGJBqIVHjp8CDu3P4flxx6LHXsnEGVUk79xSZ/vjJOX46KXX6CevDjfrQAHDh7G/Q8+gnf+7XuwbtUJuO+H29CohUWW4EHH961XWcuaZJGZBaOd3RPLKNQCc7OMtZHmAZK8l8YQmhE6LL02HSBr1TmXCsM/vJuGcQj4d66neCImuirza1Mr2ZA1yva4eZUdaoKCpaCMvk0iJJEAZ71hPV77xrfg6ac3IBEK8Kuffhgr1p1HiY2ki8pEvP0OiSBcz/Ook36UibKBeYPc/yTpQmCVi8BCadyGdoeBzZ6mCQM9o61t2Nvbq4MsVNz8aBAlW6reQLFZRf3gJMoHJ1A8cACNfeOo7h8HihW01YFEyShq/H5uVHoReeYo0UQ9DGkDNSQIhZ4U+j53PZLrj0PjqX3Ycd0/IL9/FNVIC9GggYBEDbGJGGEtFQ3XW9b/dRpcAiSKvuEIlvzb+1BdMoznXvV+pAnkiDUUYUmmGTitSAuVpXFEb3gdJlKduPWJLVgzMoRFmRB+eu8T6FlwHPYf3I/JqSl85f3XYXEb0DuwDA/8ZBtaxThK9QpSkagE9IV83vTBjiEjLnHDVCxWo9oCZI3KTaVIosmAPO2jQpsZidOufuMjYQuG7QsuaAJYQdMDGxYhuGjzhZy0uXygXtbGRc/+rlEnnS9XiykkQas4CuUmcuVJXPjOF+O+7z6MRDylmvxg7RFUgxksXdSD3p42pNo68atfPif8gqNhxsZpdhbg8cefRM/QYkVlCk34+fp7evHRv79RSp9GPauv0VvqmWeekoHex2/6JA7tmsahh+toxlqyzJEEjwPf8pZ1SCpaNwEBN7TfuGrvhUyJxsORm5cAH1+WxlKvTTKLlWjcvKQt8n5KJSN02uSZYvjxz37gnEa5BhpPyvfnUG/+Pg2Uc9MgmQQJT9U8ZANRYqE4ll3Sj/FaEa969RXoSSVxy83vw9IV58mMPed0wb6zwc86f+Nqs7oZODqc5m1cX+ce3bv1I9TtGv9nes2Ny2ucnc3NXXdfX5+yr9Dm5ecHbOVIhkeYnWJ02qW6KQJmim3oHm+yRyy9IZbvzVH87j+gDUI2rx660U8tG8Sx3/kAKody2Pu6j2Ls8G5EeMCQVyYbbsrd/HR2MmysnURieoI1SiSMVT/6LGYSUWy55mNIVmpiO/Fw0Oeg6RiF+OEmKovacOjCfpSDFEIa38ETNYJnn9uCVjSFBWtOxFvf8lY0y3l09XZgz7NFTGwMoU5fI9rHuBSYD51/N9UH38FNfRd7xxYlI65GPc61tawtxAdBAMWnYhQFsC4hH5cnd09Pj5kJcNE5/2iJpVyflWZxdnABhWJOp6zIGCQhubqfMct8p4FimdMRSzjzTevw8F0bER5voRkJMHBSGxBnCkneNr2CiyiVCxJS8M/ymZ6ZwMMPP4zp6SJyRdqj1rFm1XJce81VQCihNLNcsYHRBw4ewMaNTyKIxPHtr38Td/5gE2qzTWTiaYGXMqCnVRCZd26MCwlRfmqdoq7v73O4tu9E8P46je6R7kJ07h4yc+Gztt6mn8hgBxjRaCmaOKZlbjoElWZxgX6Msha5jcQhQoZYpm5Gs+u/xmMhtC1I4ZTXn4Qbr74SSxd248Z3vBEdXcv1zMj8EnCo6Y4WGXmQNI8yjffPf370nNsXR1navFAk9lHdZ1xcg7OzU4jH0+jKtiOZjeOhDbsR2jF8WsDFwyI7iETF9+RN0DR417f0fsg+AglPcnUSf5YEhQa9drxDvktd+MsF3bdCKHTEseTXn0e9Auy+9K8xeviAicrZD9aUPWvUk3qmjciNQWL1QD/W/eJzmNl6CLuv/wLitYrSdvPCptmtsd/VjkED09kQUu86G/UgpgiIUAxVEtejcRy/9hSk27tQD0Kq45YvW4E7b96K+rTV2easT1vXqk1m10gQWr2S8eVsNx1pnAuIG6pSKllaywdaqwosUvrbNO9gno6U4VGXq9qLM3Gdo6GiJ9tjIrAcsUTlkEaf1hnQktT9MGGPmyCvU9oECoVKE7VyE8klUQwtH8LuB3cp/Rs+sQu1cFnti6Y40lZ/hee57BNTqFTLeOLxpzA6ehjFagV/dtnL0dffi3yRQ9PIC45q3vETTzyBZ595Gu/54AfQmx7G5jundEBX8iWNDNXcqGQK+ZzNOubhVGYpxSgqK16boKgxqxK0WNRUNtM0b2hLr4lC26FuYF3UKLbOHI4/M3dYzpPqcREoisfCstvl2iJmIMojPcyc95g8qmWfaxE3FqO6KowgHcZLr3sR/ur6t+Kay0/C6eddgFC8R1MayKbSQeHUVUqx2XP+Xzau750fqV2PpMPzI7A/sOan4irTaPlTt4O8Fs3gKz/bhOem2xDaNHgqoTlBRIlsB0qFgknOPKWRBueudmWNZrpdLmZyROviuYrVMs9Amy0Spot68eTl/ygY7+/C8t98AWP3/hG7bviUhOPynvDDmIhcq94Io0p0dvkCnHvLv2L/rQ+h+PF/l5skHwQfojG0WmjwwYQ5cc82SzEWIPb3F6LElhRqKAchdLZ1Y/W6U6SxTCTbtFAr1Tz6+hbh3u8fkvsEGUnarLG4alAeUlxk0sSSxVUlFdQWAaMDCRMiELgDTO0Od9AZsmuTzRmpIhGjdJL4bv5E5NUSfY45uR0JCXa7VHuFjcBgabeBLKI8ztu4/s/8mVKtiaCWwN7pvXjVuy7DAzffJx/g933hvWhGK1h3/Hq85JyX4OSTT9Z8XSL3/sXowc1pw78bGlxGOI9Dy1PpNswWZlDO0ySgomvJFwt43TWvxUO37kYwDkSSEURaURwYPYS2bFYHmEdguVa4cf3MIhkpcGJfqaxaX1lZk1pic7rgywM//C8jJn+n7oNvB2p2kaXUtnkt+2HGxAjY0c5h6GYazx6hGG0uvfZsNNswFvG1sUI1RIMkamHgnL9Yjb+4/m34zHsvxaKVZ6IepDA9NeUAR9u4foC6aLn/y8Y9OgL7++5/99Eb2m9cHlgqMXj9AL720434Y24QEwViDTWENnSvD7hYSMNTTUKrlFodcaF2lk54l3XeALoh8KbJPqMVCBVVGu34lJ5v6rWJfuSmasBICIX1S7Hi5n/Aczd+Hodu+TXyTdZIDeRCdfSduRb1YwZQ6+7A488+g4995gvY/a1fIvjOb1AVS8Z8/MyTwOSE9Le1ifI6JTR4KvyBl6EQM08rpn46rYMYCvkiDk1MIZuK4uVXvgm18Qx2PEI9px1EPIHN59ec9326It6sSBhmcs62j48MjOp+M9shZK6MjIRcpNygpBiydh0c7AOtVkj+kEWN7HCNtxximeKmETACcWAZWxeK6AS6KN+LeajyiIsgf54G5PVGAuNTo7jk7efgnlseIrUNn/n+J1Co0eOZEc0irmcrEcEmJ3jJ0iVYuHARli9bhsULF6BaLQlA7O/tRyrbrnp/cuIQanXWcFAv94Tlp+Cem59BiCNA3QAvZmjjY5OqBz2SzoyIf9dBzpTWfXylxUqpbRN6Cx4PXGktsiSRQZo1ctm+4cNXhBb32owN+bM8ZEkHnNMtN41ooXZT3AlmJK90UdNlhp5Qw94+sZZWDDj9qlX47V0/x0vWZDCw7Cz16GlGJyKEk/ERSfb8ZIa8uZcfseMMAvzX5+t0j96oL7Rx+TZJSr8QxbPbD+PLv9qHg6UU8jVzRVHb8I+dJwRMdRX2nfu+indnpanUSu/uepmIIJPNGlDA044pjecoz/NAtjEgNj6YPTW9PxUiyRjav3gjMievw8NnvgWPlHZiwaWnIL16BPlwHcVcXS4Df/6612Pff9yN2uf+U35INqjKUqRQJCTnQHF3xY6x/IDyLk4wr73ueNSWdYKGKV6Zw0lqXALcSATCzv+za3H3Tw8gyMclVayWbVwJf4f5TBs1T3B8rarygWkw02PtAvV0G+q/8iESoCIyLKoneboBLWksarK9RNUKwaVyqaJoEwoZ19lHEppwC+yS2VxNhAfxo5kFxNkHroi6d2Riu/GfmU6VK1Xkck1Um02cdtVabNu0HcXDOdz6wI+Rr+VQKZeM3FAqKWJUa7w2ShkbqDWcOL7JSGtYBqmHf3nD27Dm+HW4+977VAotPfYY/e41x6/GjgcmUdlPIs6RXj5XSblECx8TSIgHnEza3x1ZXlMYnTCeRAulwSIYmK2PbWKTryl1pl0OBRoaMm1kH2mUE2wT2SHEDIxAIidDSPDh3Vy43pzxAIejKdWUHJCoNYOSbXrNIpYIhusqitXnD6N9aQaNyWfQ1rcMM7PUWFuGoo2rWUMmO7RQcaTv4109ZBTgkGGTeBpngRf4pxDmuU3OSEvmYTyKJ3fN4gu37sXBSgwtMtmcvluQ8PaFZwWMND6q+NrBi9z5ht7T2Gh3JiDgQiUB2tP0vCujTjFnJcn3ogiBvFoxkfhQIiGMpcM47tF/x6Z//B5a/U3kO6pItqLIizAODCxchf7+lRg97+0oRo1iGW858MrdFCmSeFNIkVTeaF5SzWYY+XOHUDttRHVdXIO9OHzZmvH8fyiUwDkXvwl33rwPKQTIF4l90EW/rtYF6zRuRn9PRHiI2Exg1V8y8HKDoV3tleXh1zCvLhFTGk2UikWBeb29PYoYrOt40wnvc96Q0mKJ1MMInCkY0de2bHqu9mUNyujMdJuR0JcgfjI8a+RymbOKmogk4lh85iDqrQp2PrkFO2Y2YqY8Nec6yefC66rUawJcKGzIFUwEoXSTwFzdOgepWBRtnV3YuWePWKvMXLhhHnv8Gdx/8xNIVJJoeHsescZ4qIZxaPSwFrgGeCkVNbYcRRfqx8aYFpcRi9hnkRjdWeYSwPOkHgM2LYVmfcznpvqVLUNHVmHtx03d092tDMhHRf4uvg8R7UJxRlGaNa7MDqoVYRlkonET8XdywwUtHrpJBL0VvPQNZ6M8sQHRZI8GmvGpqU3lNq7cT53BocwU3ctvXPVyj+xEy1r9YID5fV+vTXcBT+HRIcy/uHsnbn4iQEnG+mSlMYjYgAAZL2wbeXHg3eOPuOVTQGH8WHvNS0c1IdMkYr4RLsBhvumzZqtyFoy1dhjFuAnsQ4WM/H3Tteh62ZnYeONNKFzcp5lFjN5M+84470o89fpPILNv3JRGfGj6PHZqeU2vlTimnOAG4FZmWlw8phOhN58oK1JuFt5QZhNEYnlyvejsl6JcGMT2PxTN/5h80ybrIjvVuFisbLAHZEJzoKOjXRuP9SgXjBBOhwXIM+lIJiu6H/9dM1c5ST6bUdpGDrT3VmK0tihqtbOJEoBEzJm/sw/sFwWBnWZFogePQPvnUy5xQTY1d7htcRrDJw/juTufRiW7Xy6PRO+pKOLi5rUVCXhUqjqomLlYthVgZnpWYBrTwzotgFjr03OMNXCliVe97rV4yxvejg237tF9YMuDP2eZSRy52YIimqmOSDYxm12+uEnpq81SRBvQtXh4nxhd5C3teq8G2BkPXNarLlJZL5jP1MQwjMw017Nsy4wX5jJAx0BjqcFnxfKEG5iqI6HDySPOjmxTMbKr5xxUcfHfnI1qbidCkTjGxsYUxeNzRg4hOVZKoupagnMbd95UvheqYedHWz9EfW7Xa5hACPFwGN+77Snc9kwUJXCOFdc3cRG2FNxUBQavrSNn6dbyhPSsD90cpgNucpolzs4lj7rGpM1Z8SkB0zVK9bzJHL/XR27eXJmTs8XkjOi44Gb6M1h255fx5Gs+htClAyjEq6iXa4hnO7B2/YXYd8nfafFYP4yxVMN7TT/nUi6lzrx9Gi1CtQijRhOz/XGk30V+KQ8Ja5moppRWs4WXvuqNePiX46iNRWWA3ar7mTVO9+lGPnpvZAm7nY2qiFBCZ+0UjbvBZb5u44LgK5+flSKFBwY/G+1R6FAoET1PcEZS0hmDBhJxo8vxACToVasWHUHAeGWemM90sVIqggB0nGCca6fUG4xGtpFqyQrOuvoMPPZfD6PRvR+hSF2icrW2NPLTDiOPX9Dojv9GJL3WYFupLHF9IV9GKpm2A7FZx8x0Hh/9zKex94kyigfokUUFFrMB6/tycRFDkClIKIR8IW/SPi1u1pwcVGZaaoJ/Att0CDclJ/REFAMIY2JK8XkzQs6NJ5GayGYpMVK3yd6HaqmW2H5ztq1UshWZ4em3S3lktrgGRumQndNEM7BwwqOVNASeTvzzY5HoqKGSm7H+c5j4gqXJfLFuFxg5X1MrEc6RfXIk4DqXEx8C5xE25iv8WFLSNfPff70Bv34mjCJsrcTTZNORLWYZpR8eF9rYc3LA09AMoW0atxA3OeVruzqswT4A00XaWTINlOxOobuFbJL2KO6CONfU1QDeBI4nlOxbHMLXjAJDt34K9VAE93zpn5Bbau917LK16GyNYPz6T6AZNXI6HfbpRuBPLA9iPH/jUulBW506RqNVjHz6KiGkRCzllhCn1I0E+G6ccM6rcdf3n0a4FEFZg7isxmIbQ3QyotsyzQtEVGA08MwZ/hvfkwudJzSjH69JIojACAdMq9mOYOQiP1nc23QCcQIsLomSGUA0JtCKKCgpkh2dBnoFjaqzuXFSSXGlWQ5w1CZnzNuEO3+qRyIJ1BsRFMoVVCJlnH/92bjn+3cjMjCGZst41Hx/z77hVEU9Zc5oKpbVj6a/FFF7L7tT31JZQFP0R0ocb3j33+H+bz+HUDMhk3v2Ejgnie/L665UicQbWMfsoVwqI+nQdT4rblzrf8esNUPVUlsG5ZpxwnkPueG5oNva2sWA8tRTH42pIGrvaDO+tiR7jpghpxRuSOvTckPzuUh258zluL6Zdstt05Vclm14bjTvdxQDZ2Sx7JQFGN21RQe06vK4Hch8sa999MbVWpy3Keei8FEDwPxmt5T3iKVxKBTDfRt24yt3TKPcjCOIJBFTOUXTQmarRGts6IAyjyc7Tgj4ZppNE2f9YD001miG+pl3lOeYdrV3GE3Mp8H+w1Ijqj4oVTd2sZ4RI6GAH1btEDf++8xZK7HiK3+Pu6+4EUuvO0tCx2imE7nxMCbe83lw5LIALtYMtGadP/xXd8YAGlvUNiqF59JMpIWRz74GuSb1oLSBsUHJBHrWvvjlKE6lsfn3OQdImSRLvGOe2hHblKQ5cm4Q74e1dBghOZg6JldFLgJ+tpT4sG6siJvVyo3O+iuRsJaHShlXm8TiVtsxE/HaXKavRHipWJLXstg/bqj2PMCPN7ZWLStdZtS39w6bfVCLA5lt0PXZf/ki/P4/7kHQNqrIrFlznE3sRlkq13QvZlpGBpkHqBCwcUbiPGBKhSLOvOQyFEaTGHsir5q3QsM0URxJj6yq1ODGK+TN5ZKbiuQNuqIoGsq5xMAskUkCAmt2MDPSsW8tRZUiY0htHbqtGLBjBgV8ETnmNbJONiMCo5YqC3LtNJ/t6WASVdM2LJ+HodUWea1OBcLRiLILcYJCYWSHozjpVauxZ9vGudrUYwsqoZy5ok3Pc/fS9+vm7qwLe0fVtM9Ll2WPQ8JTA+OFMt7/9WcwjTY0YmnZvsaTaStnahzknVLGJC44p2Q81XWiM0Q3obv6Zx0dRn9zhm1EgxkxbWK32/FuQfkPwtOUp6IMy3kCayMwzXKsK9/2IJWP/rlM26IxDD/0Zez53I8w/qP/Rq1Vw8hrX4bCypWY/dBXbFzHESbY8yKubrxQYEvNvCkbb2YhEmDBh16J8SS9mDlBwMjvTCXPufw63HXzZgTTxkGm7pSfm6AUr52pNFMjfj91yjwRGAUZOVWXiLFF83i2j5pIa7KCcZe5CZi+8cAiwkzrVxMb2CEoml7UDjQtGNIDqUHVbCACfexvhpFgy0N1HdNJ+zPbavx3Rnv2q9lOESOI1y7taBLleoB6pYYX33g6fvuT2xFvnxQophaPi/TKkhzZRC09j37O+R3bBvYHN593pqcPp5/zMjz2090ojfMwS2rDMjctFug6QbUUyRpGCzWBe0g4yMThMRC447rm16391ZKUL58v6B5ZKm12M6xV+Tv5M1QCMRvgvWPKOtA/oFRZ6bHsd6lAMvDR9RVMyOEGirFNVMznRBflIVcu0zzO+uG85zyQxZVWORZGPEWqaAiteBHnv/VM7N35lK7DJKVO/0uket7oy/llpGM8Wp463+rC39v/8XWKM0KoBjV86N/uw9ZiP0LRhCyBSBhiek5ar9cQM4Mayi8AACAASURBVHD4/n7o8bbj3dawMYEecu8d6AOn2NFipCWWiKUTNr3MwJP5LA/Pu+SHZiriN7hpR63Z7Qd8MdqwtmLU7vmPD6KeTmP3pe9CuVZE6sozkDjxJBz84JcYQp8XZeenygIH3M2xtMXqRG6uYqiF2DUnAauHEYmF0ag1JIfqX3wshpedgSd+fACVotVdOmxicbUU+F9+RhqU8XSjAIK1kjX8WYvGEecM4ahNQVdLQYivqYh4f7gQWA8z/ybwwtm1mjQrX2PycMNSCvH3UnjPeyiuc5P6XLaEmggHpmG1iGoRhx+CRAmZYmtUhqWkXLg8kCKRpAzDOe7mhNevxR2/vAPDi8M4dOggkhzWrXLAMhih2O6/RsQ3FFbAm1hJtBgy2ilbOC+5/Br88ZcbkKkM4sCBQ2g1w2hv78DefYY4c/FyNhDbJpp84eieau3EEyLaGE/btMncJnK6cACWrF8jvNcFpBJsz9nmdbOrVfszI1HpIVDpyNgSUj0ZIFLCFpyxvxu0RrklLXA9+433T6YG6qNz/ZgjBwk/as0RJ6HzZrSC8647DQf2PWMjXnTY2cYV8eN5UfVIXfv/eePyXYMWfnH/JvzwwQaq4QSiqR5UmUlyJAoZhRHXVmU22QwELioDfaxjrVJlnbIOWPC6UD5cwuWkM1LELP4ua0K3YTwyxp8X7d59nYIFRh72Dr1PkC1A9z38PhEammicuwpL/u0juP/E1yA8PYP0Jacifcm52P6OTyFBL2JWdPOr+KNSETvdDF22YhySHx5a2YYlbz5P/s+ZNDWsJZxz+TV4/M5DKOyIiNHj60RNkBdgI4K247Ia+ql6goAK5XrqmyaRlIuE/TsF1lwwMioLM12kqZqRBIRiFktO0sfNwe9rU8bBk7PWrGGQ/Vqi8qRxOiYQf5cxpgi6HfldHVk7OOXCILsX6wmrhaLISxQ6jBUvX4oHHn8M0ehhbRIt+LR5J/u02DOUGHXmUNu6SRB5bcl4Gs2ghjMuvgxTO8vIbyG63kJxhuBVXiwpjprMF8qoVQmaMOMwcYGuwx0MJP9zo9EZhP1gblBD43nomEujPzQUTWS1aoZwJflzWUTm/3VfWTK5mUMei2C05+EkVRVxAL2HqYy4BvnyrC2NQdGAbluLyniSJlAnZkGhCbW/p752Ncan96NSG0cmQ8TbXprV67IXre0/6Xrxv6fKvE/8/X/9z/dgMjKCZrwDkWQbYikzDPC8eR0YPBQ5z6vsNOKPd/iIy2fmhNw6fY1Lyovv6+5BoViw2oSppXcnEDrqDMtdW0ZjMmUGzlMsKtXR3CnvLt4saQI0edGpOIbv/Fds+dx3Ubz5NjRWLkD7e6/F1jd/CMkghBjra3kWz+uXebraUTWv5ztXwsD+jhqOed8VCBJhJIMoIp1dOPn0V+DJ2yaRHy2iWm0iN5szBNNZXwpwopF7vaE2BFsE8xk87GfrnrA/rAFeBHNo5Ba3dNctBuMTOyvSRl1ZC9s+BFvk1FGyOpAiek5akPqFcj5FWRN80J2SiziRosVOzSRt/JqrRTV9SYveAT5kXcFqxkUvGcFMq4idW+7X93PR0ZXCz/eZnx7z+0WcbzblgMHPxgxgejaHk847D6F6Gvv/MIFIPSHTuVYthG3bdittbYU4gnQXopGEEHxrCxGoi9mfmeaqN0y9ctLRLW0DMt0XAUL6VcMMZLimdLklVNk2vVFRBeD5WtlpWg1INEsfIueWNFgLju8ld01xvK1lqM3A9l7NLHI8QhuX8ZuNFCEQ19HWg0Uv7kX7ghRmcns1cdIfEqZimseWcp9Fh59b38+PyPbF+dkp/+4Pt3/+3u/w0P5O1OMdCGe6EEtl5iZ88B1Z2xPxVgChgUOFf28h9Ejb6sDXUX7jGo/TtTvicaGfczYf9L2RiMAr+e1jegIGHwSlbGYcHAicmGs/zAOoGEWJTIrc/433IGhPYsuV78Z0q4Ghb30Qm1/3fqTnNi51u4xiBkZoRIpP1d1dkvLPAQTVoIWpZB0LPvpq1Dl1oQJc8qa34rHf70NuWwSVnOmCebLu3LVThT+nnIvW6HymvDO9IZRUBxlARy4uox2vV6AK7T7TSUOsUwkdxroHHIfpwA5mLGQv8exhROSIjwUjI4rKjIZKT1kvp5lq07mBdTEPPJYTbIdERCAgiOFVWWzHqD+udkkY8XQalQp7vTUMnDSEjmP68Mh9P7FIQ9Sb7RWX9YjcMEdpZWpL8zue8lb/cqEsWbUG/YvW4sDt21GpxFDImWEdSRbbtuxCe0eHShOiypOTMwIAdUjI8tV6+Hz+smGlY4WqbE9RJJLvNhR7Ww4f4PuzfGCqPDw0JE41gSebD2TPXGmrR9ndIC0Dy1ivRtDRYS0i9qNVwpDdRkxBLUT7/VxG1YoRghTN5VkFHTSck8T+P4arOOeqc7Bj15M24REUY3BihVbakbxv3sb1KPH8+bj+G5+/ce2zTE7n8defvRulbC+iySHEO3oQTqTkq+XZWsQseD28JyySWDaICPpY+1pRoYSMuk3ATcpThjeSi4kDovUglJPbtxmiduSliepO4cHL8ubbjFKsaZliqLZxvUfJ+Pyg31ecjp4Pvhlbz34rytN5xL/0Djx04ycxVA+QDMJymHy+K8SR3+3TPP9J9LCCAGORBvrf83IUExFc+sYbsWdzGeV9wPjeaZRmK4riTDX52fI5yt2sXzjf8Iv9OuPb1sQlNufAqA4RXn+jWlebhwuMt49kACO/N5Ei4YLvx1kvmixvaHKj2kBnZ7tmACnFdQtSelJuQIrtOTLDeQlzCh+7SBwh4iWbirp8RhRjiBLJGpqzY81Ct2tJB5acuxz33v4ztLdnMDY+qgXPQ0GIrwO1rN6k+39R94F1KOvyxWuPx4LFq7Htrl2IluOoV62VNDtDA3Nayc6qFqQgpFLiPNy8XE7URZiHgTDWx2XH49a72kQlJFPcyA6s0wRHZiFFHXgExej04QeS0xHD/L8ccUezhoydxmyF7SYjuqS12AlAGYWXkk6T+lk5ZWNMxCngoPZy3oz2SfaAlYTm11xGOJpANZHDy996MXbu24QIsQcX/US6cIezJknOYz/N7YZ5GamPrnPMKR7dQQQ1FPH+z96CHaXFaKQ7kWrrRiKTpZWh8ebFt7Y51fy83LBSvIt33kLo0bY1AReAPoAmk5nxFT8db4D6qM7sjQuGkUX1kRM4z31YZ6XJn+F8VR8RWf36ekfpgbtQcoz5+/igC11JLL//G/jjyW9BtJxD+IPX4OEf/QLdG3chQ1mRU8b4lMPD/fNTEJ+O8waRZjlD5PDqM3HBh/8WhcMRjG2tojLZwNRYDqV8WVRJ/n5DM9lTY9O+qEXNjapF5IyxCckTxWUNZKQLDgbjTB2SPuhRZaATWxncAOIic8GyHUGgq16FbFZLrHfTKBbzyGTpF30kjWMPkveG70WKKP/Mz9Pf34NKuYAoxeHsSTtpmmHJHnCiEiYudlS2pxvVSBVrL1+Lu371X2gFRW1wwzCIskfmNq5q2WTWMopwBFXW4/1DOP3sl2HTHc8iXWhHhZMWNfeX0+Zz+r6JiRkd7FR9FQrcPBmMTdA10iOwbuCb0n5D7bmB1FJEQ77RJPHMIa+thq6V6DyRaNXicqkwxp0FFjusxQtw3lwUshcLeSxZskQOHbn8rNJrk05yE9YklhH45gCtufQcRkll1pRMpw055gFCgCybQTKdwLpXrEQtWUJuclxRzrO45rfT5kfU+evyhTa0slRRJFvYO1HEez/3e+RTvYi0DyLe3ql7yhGyxEq4z3h4kdg0V5p6A0K2g7Rx5/UhFcHCIWRSWecAAelpmRtKl8qr89P0XJTWLRU5w/yAaChmG5eGcZY2zQey3BGoTaCaJhxC/+PfxrPv+ypCv38Q1QtPRLBgEDs//210BMa+YVrpU/T5ULscMlzNoNRHtUqA0fY0rnz4R5gd48jIJqpTZRTzDVQKNREt1CYi4lksoFY1hJu12dT0jOor1U6OTEHqHxegro3v3wo0c4c3lRan/ABsu5ClxZ9tb8/KwzebSqPM6X01MxqjQKEldhI5zDVkM6aCUZSNmhOEDkeqfep1ETJo2VKv0nM4g0hg/VF7mWeT6JMNglQsTyJo6+1BEAuw6IIleOD3t6NQ2Kvszpz3HVVQLRhLr8jt5ufN53JoBlG89MqrsfvRPQgOhjXcKyAWI+8t/r4wxsYPC9hjxC2WCxJ412stkNQhOicJDorkloILMkuQfEJDd0YOpsI1lUk84HhPNc5FKbbp0KSskh1QXFHUDhbbuEqXiTxLFM9B3swSOJmPkZTCBJI76PJovWndI9fnV8bnhpyTK82+uRhbLtXUNQZN9A72IhXN4GB4B172hguxY8dmtBzpQp/BaafnJZxzSL3/2p/auBHSGMMVvOPDP8b+6hCa9NNuX8j+lAbhRTkyJWjo+UsUYnwoHboq4R3fPPTH7vU2rc/3TENAxk2Q583wqiBvVmBpsOtpsYaRhzKRX9azCVQd2VunrzyUjzT2+TVvS6NI7m1IEKDntn/C7L5RTNzwj5g5pgMj734z7r/qnWgTTzo8x31W9J6nyODpJ80sca5mCJF4EqUVwzjz11/FzLZZjG2rojhdQatCTjLmVEBs4NuDYl1IrS3TVqKGxtFmCspNw542U2qe7qxPeRdZs1k5HUYg72SysxpAqIae3m7r04aZ7jRRnM2jUa3pfYylY4boXNyVUh4dnR2OWM8WEAEu1q0G5hABZcRhFGcqVy1NC+Biaklmm998rMslzaRRWob0wRgGTxnC/smD2L3lXsR4T0oF0fz0DIRZmFhE7k9BIMLDqRdcgsl9VcxunEWrGUWjbtkXgSd+D+8Jx2hOTZLOmEalYdI5sqyYqXhnR16bZ+MxSjEFZ9sm7GprRdGgrpqfhndsLdFjir+D2YznePv2ju/zsg7394UKNQKWTCWJzAqoi1prrZgnSYTtS5YxBMmsDWb9X6uVNamwRc6xMayYXbFXnMok0dPXp2wzlIwhtSyEodX92P3cs3P7lHdlPt1RmZ+TnM7fzD4jnL+ZqRLPlRt404duRS3eA3QNIdnVg1DELHk1b5qqrXIVFWpxnTrPPMiNjCRA74mudQFbPV5/amSAiJBQf8IJineWH1IJemDDzWxlOpJmisOer+PB+hPHD13yOb5aTc7RXmCJJHlNRD/yJvS84hxsPfU6zCYaiH36emy89kNoZ/3BZhPbDO4OzHfNI9fYUENu8Dj63/QqLP/oDRj940HMHGihNhMgny+JylatmBsDwThGByMNkAVNdJgLs67emYjqqseddIw31AEDAnpkpm10vHTMFod6oFHjMGeyaU2J54FWzOWRcgQNtUGcn5babBznQXJHMinU2ZBGigxicswgiKWSLmILktTPUiWPVMKQZ1uMRkLhwoln0sj29yGZaUMuMYv+lSPY8OCdKBbH0Qz53nDY+pVCV9kXjqKrqw+9CxdjyYqTsfv2XWiWIqg2WC4YEBONxJUm+tJm755RFIs1AWIqNajGd3Wn6WTtsOZPa+qiy6zI4ZKsjiUH6+NqUbUpD1HyibWhdIBSxGLiDF8CMZVmr5UgV1+fs/LhweOnHaCltptlFWzVmeWrMees9UPChge4uI6Z+VCEQracX/8dnW3ydeYG6h4YQD40gzXnL8Xk7CgK+cIc3/7/tkGP/rf5GSIPi4/+8y+x8XAK9WQPIv1LkcykEAlbf5sBgPpgkZ44MJ3llLMx9k4hyoofyq4ShMyaw99Unpysz+RqSEcEWY2YKsdL/GxhM4Pmmc3hTil9wdtk2oNjjLf+rU9plULzEHCT+PRQww1UXnseFr7rWmw++TpUQhXkPvQa7P7YN9Cey6MrnJS21r/mQBqCBOoXEqKOY/1Nf4vsay/B3sf3ojya4GhTFKermnvKVJAkAfZR9dlbgU1g1xhMmyJYoZdVJGY6Wk0WbJlxma7bXAVlqeMWgozO6GZYMmolPaVYLDdaDSTTUd2PGGvuitVpOvwcOV2gX5MAldH9eAncHOSB9/Z029eUHpqti6w6xVclH7hoKiHH8GKKzjIm3dmOZFc3IskUplqTWH/Zi3HPz25FMxhFHeYVrc3EfrUDClMZaqtDuOBVV+K5329FZDYjsnyrboohEVuoruKCcnYt+/eNoVZpIXC8YJYUHELNtJb9XRJY2BbiRbOG5DPnPeW0Pt4n8pmjHGdDQbyTQpoai5pgI2NISJBg5DYLVqbevF4OaWPrTAIQaZ15z00QQw6zhAt0Z9H9s/6nJ7wwhbbpBWZFxI3MDS4mnzNnZ4eAJ0b/YD8yvR3ItrdjOnQIa89dhmc3bTK85ihgdn5Enb9Jj3z9SHmTL5bxtg//GuVIFxrt3Yhr4yYRallbj59NGAvLDreRVWaaBGpOlRb6Q/a4INwMxHAhsVtjDtwbWI/NHDD8KardzsqFUdgJ23lj2K8VgVxjJU1+NHcRrhnvEWBGT5uT6njGYaD4kuNwzD++BxvOeBsirQam3/NK7PjBr5B+bqeIGElK4o8iYjDZI8OnFo7good/jOnuXow9th+NQ6y/6qiWKJCvKYKZyDqEsbEJRa9MOotcPj/3wLiwGFIqdSpSDBDwNa2RFdiftHTQj4vkwZRxSKoiIiN5g86FIRQqeWRSSU0baDW4cAsiVGh4meprHoYG8vFwjEu5VENXV4csVxhdpL7yWYbIB25iBA3Q6JkrMQhTRANguob65bEc72hDvlnB6kvXY+NtT2K29hRKTdO+MrJwceZzeRNJhBN48aWXYXpvE9UdVQTNxBwrjNnXxMQEUumskUTC5B/PYuzwLGZmiA6b+6OymCjdUdiSMqSejDMePJRCclPQ7jYSbpj3kxsKRyIE570QFGP7i71vWcs6yx4Oqg61YqiRvNHeISdPKqlIE7RgYmUSnxXpq+0d7Sa0JzPKbQCapPMmcrPz655oowO71ZS5O1Vb/LuZEpSwZOlSSnWQ6uhCRz9/bx1d6yJIdWawc9s2M2dwr/nkIGPwuTrd1aN8fja0PYZGqIgf3vIAfnrfNFqJbqB/EVLd/WrFeYop12mZg+LqbJkRvTVWm2+1WXkUIHR/emVAhDTLiMkERpvP0dJc7UtChbXx3UtpGsGKQBFCFDU5CtjPqz/riezzkGRFXg/Pe8E9iRocYbl8GMM//gSeeek7kZ7OI3fNOXh28yZEf/MQkty41CTOO+l4AfT7zQ8P4OX3fg+VYgj7Nk6iORtFpWhuG6V8UXUaWU2cK0qQibYoBw4cUF0Vo4Y0n3N0RAOomkEIuTxTKBNu8/uJ9Eqe6MoA7h9S74g2p2nQzUhCgCkW0UR2kQUoJ1R0toOPQAgb/7EwXS+Y1vMmEtU1twdyFbt7ekVW4Mb21EDWfOLSSs3N1LAJpZxBzTjBXIAuemZ7OpFqzyLd04uZWhHHvXw1Nv12B3YfvgfhjPVVjW5qjDA+i1K+hD+77u147padCNdZY7PGZAlhdZw43rwCN1FgapKSvxomxvOIOg8ylVQsr9wi05S5OMdC5uSzxfvOdg9TwGQyjmicQ62LaO+JINsRR7wjBLb+YwkbyOXBrWqJnOwQ8lNljO8sIKjE0ZHtEoLPZ8MsTx5ebl3E4sYnlxJKHHlnbyNKI0UiVuMqnachBANGMT+nhOOa4ubPtmUR5yjObArJ9iw62zqwv7ATJ1+4FvtG96FW4oxae70Qq0+HrV+rag2xjRpDNWjgmnd+C7nwIKJdi5AYWoBwOmsB0GU0co7kYcyfbzAzkPRBb2dSTPtz6IHscUFc7o5E6szIWoOU1OwmeZ6nnvOfFVDBm2FvQhTZ80WYemiPUq6mVMcTrT04xVPyyER6r93VCcULWzSIgdv/BU9e8T50Pr0XB4fbUb7qRdj7ia+jB3EkXQtANiNKm0KIrT4WZ932PUwcmsL45gaCfBPl2QIKlQC1EoEd1l8t0TW5mJg+8b/9/f3Yv3+/wCC2BKjh9QcNPYRmczZwWYR1Z9BNhNTYYIZa8qWay5P9pQnmQC/WYmHQrpbkCD4QuTbWyygUaPNZ0MZRKhgmAk35Wgr93YP6XUoJo9bP5f3V/ReHmMWujafsaqerZkk6WRrmqSInMb+nC+muNqS6ejFZnMGqy1Zj6x2j2Hv4IbSSs4rMSiFpuCePYfkE4pVvvAEbfrgD0RBrSBJcmMITLDGmGK1x1Gar1zE6SmF5HHkSMlxfWCm02xCGYVgLkJuQBxZ/doajRUJVdPSEcPJpK1FJHha6ykgd1JnCsuZnVmStOLskO5RIl6zWSggV4sjtD9CcjSPCodk6LA2TMRqkyfr4u3mdbKsxS+Kf5UDikHhGZ6EWnK5YKQv152Zgq4n3PNOWVV86mY0h0zOIbNaR/kca6Fnajp2bDagSc3deFjg/w5y/cWkvzOf0wB934rPffhiNRA/ifcuRHBxBjPOZKXap1hR1fe+WtbtIR9q4NvpGskQCoXzuj7avkVmcB0Y09pD/88Zc3MBC4MypkOCTX9BJkbINJZ1Le90i8uGdC1hfcj1Hf1IJn3Xu7GFuhs4khv7wTTz7l19A4vd/RK09jpn3X46n3vFxLAyldcqKG8rFhhbazj8DZ9z8BRx8egwz2zn2gkSHGiqFskgObF2w1tKUPFqQcpaNc+XgZzAksSUHP8q0eFp7WRcjhTX46WVsKhf2CT0QRP6sjdZk7WtqE25GpuIkSgTNKtCsYHziIA6P7UGrSVqj8Y45aEwAl0tvfUrOKMrabu2q1Wgj9Y0T72KMTsyE3Oneagjt5M8kOduoMEOSI6wCJEDZj0gmgUxnP6ZLU1j1yrV47rY9KNXHsO3QHxRJGPHiSeqAC+aK2DaIc/7s1dj0o902uM1EgIhFDeXkM5+cnhJnmKf9nl0HEQRR1fUc68Lv8SojXwpR2ULQJxRuoZDLo9IoAdESzrp0MULxCkplTp8iDdR5kSkS2ybTjB+3YjSF0bVodM81qK1FwB6TW8qY3E2ZZVqZUyxpkxRMKBHRKBJbm6wbmyIwZNNJJ6yvzE1SUKrfqAgk0+cPWujs7taG5AbOdLQj2dmGTCqB8doMjjt7IZ579hmNnqFAgPZItomPjI19XmboWqHEC97+ke9hX6EDQXYAyZ5FSPQPWztP9jQ2zbBJphRH68kS2Ea3KrJz/zmaqOZXsR1kIdhefuMaN9hFUaalHIdAXqy4x4Ta06hpSp27za6O9Tm+P32YJvq2j1hNDlnVUe+yb6J6QTqKkYe/i22fuxn43h1oRAIU3nkp7rvpC1gUTyJFCy1ukgBof+mZOONHn8eWJ/ZgZnMIyHMKm03N0wgWWo06ckc6lTErFkYFprqMUAJ7rN/IBzo9M6u0j0R9LhS5J4gDTEvVrDY9oTZTvxiSy0WnVlmIJQIwPT0htLRWmcGh0e2oVui95LW6jkTChe7wAuPz2n2XKknjWCxapBMJ9HR0YXhgELFIco622Nne7iRm9pQ4lDpUr6LJD9BsoWfBEOIEOtJZlFHGsouPx7Zf7UEQrmDz4TvcLFoqT0Jq+fF6lq04ESPL1uPZn+zQac5+bCQes7k/DsvgY+JG172aLiJoRjE9My0JGg8btnr881YrTBGdhJUois0pLF2TwfAxMc3z5UahAGV2pqCNSnosQTmLKMYFsJ1gA+CYYfH9GX0kDuB8JqWTAcLVAPs2ziJR7UciltIJyufFSMu0XVkUsQoZHJCBZsoqK/NsM7PmJ/PMwDSzE+7o7tThlU6l0N7TrZSZh108nUF8pIH24Qx2bNtCtficc+XcBvKbeN4XeKgWKlW89m/+E610F0Idi9A2tBiRjB3CygxbTdkJMftgYOLn8BvX6lsCwQZe6faQq+zLUAJGXLB82QLz99CRLxh9CdK4ERGs0bRx/ffN5w97JZDoeTbvVfWFK+C5AX1KxHQp2p5G3wPfxN5v/BzVL94ix4vZl6/HQw/ei+HRKYFT5PDGertx0dO3Ye+zh3DgAQ6RLsn9QRPxOHCMzm9y5LNeq6HFjIaOteX+K3MA+hvXaihQuscSAUynTaxsfWabycpFxZRKG52nvqNqEgCxYV4VFArTGJvcjlxuDNFoSbUsDztzEfRAHVHmhA4Wk8+ZWJ7fx9Tf92WZsnGLE7Q5cc16dLZ3akGypJnjG3OiTSyCSiEn21ue0D0jQ4gmE8j29qIYKmHx+Wvx3M93Ip2O49GdP3KsI0r1HJMpaOHMcy5Ftd6OQ/dMqHXDe0ItrMBHaYCr+p1cXASYcrkKWk2OSikgqhLESP1il7l5wXx/orV9I0n0rS6jgSI48jrOrENItKWEPH4YSTWyhemiq+FMRWZtMHlVsf1IYwORNzjIyonvqWEsAwefmUayMoz2bLvUXRp/wllURLSdeICfrVLMI8t+OAUJ1G0X8m58qm1c/wwSqaTKF9a7HD+aaMugb3gQyXQbirEpLFzfh63btiFoENC0XNmDt3PRd97GpQ/yb+7agH+9dRciqXbEB1Yh0z+MkMa2WgYrT2sGQpJeqBSThxZXvG1UlbH+0OFvZTvI/1IPHPmNqwPI1Vi+t0nXRAIc6q85frLjSgoplkcuh/w5SF/hqNFU2id82zevmQp4PW2oiURPL3oe+Bq2f/6HCH3ndpHQ92YD5M9YhsKtv0M2mkAmlMBFj/wE5e5hPPGzLajnaa5dUCQ1T+SQasbZmVn93YvGreHvMwNbENq4nMlKI+1GQ/pgO+VN86g00bHImKKz7ufi1YPhYGMuxXACjWYVk9NPY+GiCvbtGsXE5AxCQVI/y2nsJHZQKKD3axmaHo8yRbQ+qWxjqVt1Nj38rASkGOXVKmsEOH7ZSiweWYQ0hQCKGrZYWKuaTM1cR9p7u0V5pMKkGqth6QUnYNOtO1VH7pq5DQ06BfIwSiScD1OAi175emx+chTl7UzVLavhYiLoM3/zkp9D5PHRVAAAIABJREFUp4tcvozpmYLmB0UTJikUGUGWrNaLrdfLGDwmgcXHN1DWfbU+Kj8r2WNjhw/bHF5NKgirPqbeli/2a/nypQzfmwyzYjGnTcwoqbajyjP6UYeQL06hsD2EcKFPw9nZzlLa67jEnhxRyuc0nEwRu1EXXTKdsdGnxFlY5tS5bqIxOW0wE+jq7UE8k0I004FkNoV0RxI9x0Yx1SphanTP/x5xRROu4/K3/Qtq6aVItfUjGFyJNg6n1oFYM3koe7bMwOTNZg40Kj/dxtWh7sBiZbX3pldwjTk5mZ8DyzEVBjSJ5jh34+tIsX5xUZmb0TNSlKI69UlEnEurYUXgTiT1gVpMK72W11EndVqFm4iuWobBX/4znv2LTwH3PcUGHKZTLTSuvxjPfeZrGEAaS//i1Vj7ib/Dk7dtRTCW0DhGtgE98drX2uS8au4YUVPnhC/k1dXjBKV4itPxr8wp8tU6pmdmdMKSlEEiBvusTBvVxxRbxaKELTQ+3Aha9SriqZ1YsaaKeKgs6h37wKGA9izk+LaQmy0hXwyjVGggN0NeM5HmrJwWuAClG43aOErdC01+sPmxjBocaBbUW1i3fDWWjyxR+nZk0XOBh1Auzmozd/b3ItPdhRBTxUQDx1y43m3cKLaP/xahFIeQtaHWIEhnM3hect4VeO7RA2jujaDJFoizH6J4wlM+2XfloUX/KY7YlKkc6/95jCRiEDxsuB76FkcwuLLGjrMOAx70Skk1k7Y213vl/UxzfKfAIS/xc5xkN8VQ3YNoTBY86hfX6PVF0X1Rm61RrqERaaKVr2F8WxmpSj/SiXYdJH4kjieAsF7kpA4uPTL8GPm5cYlTELASPiFyjQFz6jzEY4hlUkhmOhGKhdHe3YtwZx4DJyzBto1PooEjE+xfqIfLzz86lsd1H/4ZWul+pDv60eo7Fl19vXNBguWD8AWJC1gyEFU2uazfuPwzywWBpAQA78uulJ28UkOnqVV6Ic8hywS0eF2Pljas6sM6cMk0kVxczieJKhcOfXL0LEYTpteqsWWK5rpg82xpIpEWkte+Ah0fuR5bTrsBsckZ2ZYcStTQ9o4r8PSnv4W2/n5c9eB/YirfwrbfjKFUrDvU1lJu/39t4oYhyXxgU5OTc5pbXrCoi06ozfEOpUpF/5eLgxBiM8uWVlOEdZvDyptpaDqtJAJUC3n0DBzE4iWHETTZNqmiPduN2Rxnu9L6xc+9iciZQumO0iCgVongyae24YktE+hsa8dLTlyNZokzm2i6xkyag5pJajBTOKLe0SCMM9Ycj4V9i0w8r/voiKxNa+/0DPQi2dWJVjSO1EAWg2eswDP/tVXSuP2FB5FvHNbnIPGgs7NLm/HMc67Apkf3IThI5NSyFAlF3JgSHrTcdIVCWQdaqVzTxuXfE1kDznjYJZIRTZUbGGlH/6pZBGSOEbRzNjOkKNKOtlgqOWNyox1y7dAi1jIih54T4XXmdj4bJGupq6vXlVvUKhtphob/nH/M2c5BuYXn7plAX2IREsk04gn1H8xtRAcmMDs95TjMpgcmWMcNzWyBXtcCKmNUxaXNtYMlA3vA2XYh1vE0dbMVLH/pWmx9+hm0wjalns4f86eRKKMTs7CFH/33g7j5rr2IJPsQ6xpEZuEKRElEqVudTR67zBVZvzpCkApW9YCspFBP33GWVXrdk12hjWtOFRSJ/x+q3gPMrqu6Hl/39f5m3vTRSBo1ywXZwtjGTVRjU0LiNIwJoYQQev0IBPhB4pAAST4IhCRAICEGG+OAMTYG3LtwwZZlW12W1aWRps+83u7/W2ufM9J/SD5Lo5n37rv3nH32XnvttawuYA3qT1pfixKV5cnqeZpsAfFLBAUCGX70jyAP0y0BWnEBWiJza7jawAcV2g4Uy+Qy6PvJlxA95wzsO/c96NRrKHebmE220HzF2Xj8jofwzs99Hqs+/Pu494YtyNX7MDs7pw+biLnUx2kVMT3Se1OKRKLYRn7n5vMsMNZJfAisfSkOzrqWI3yk+Rlf2EV/vpajPXo2D0+JRm0RgwOzGF9zXAymUqlPXrOdjk1+kDRP1Jd9S35e0tZMo7gpggGnkaq1Lr76P7fLKPwL73kjwghPd05MBRpW57V+/8e/QaXDnzcw7LLz1uOVZ12OgfQqaRTziymjSc+GIm+k+0uIZ3JIjuTQf8F67PjZDkXo/TObUQmPazGTkNKhtWqng0tfcw32PnMCtQP0ljWmE+vpxWpZ78kFz40eCeKYmpxVKsnsl6OQQeKUAiiJGcm+EGs3NrH2jHORTvVgenIOM9PWDuLaq5TLOn0LhTwGBtNohgsoV2cwuzCrYQRpKVMhgzy5bohMIq9WDlUvyN6SxxXLB9jAvjIWyQpZfcxUONpI4sAjMxgsrUSUcEKXabOVaKJHkuBQLUuQ3VRKzKmDLadMljW7lUNMlWXyJVO5KFJ5km8515xGN9LES996AXY+fQiRxFEzaydV8zRzavKyaVVCpdA/ec830UivQyw3gMTYOErLlqPO9daoqw2kCTKK2JGYQvqoJl7dUEVomIuxELl5Q2sx3ptbp0F6r92rGOXsG22HGVDlGSB2ctqN0Hcdw8hrTqmWc/Uv0zqefhKdc8HBc3XjolDyRnYQFNNYvvVGnHx6D+p/9i/oBB3Mtqs4HJRR789joieNq/78/TjzbZfh7m9tRzxizBzJvTruLxehGDzauB0QgeVJQRYUjckYnZleefkWP0RAqp4AKfYrG3WlRwYYtKVswd83MXduFPZ7O4iHc1ix5llE0EQ0QdkTU/zgzK6BUVZfhQTMmm2107woPE+raDqOaBjB577xE8SSSfzNu9+IpCiR5nNDKR3K3PzXzQ/iZNnsTshsu+jMcVx+znqMJS9AKk5dq1Ou6gzHHCLPDfUjwtq6P4mxTedh283b1O88PP8kZhp7RSM0CZ60FEAuedU1OLm/hoW9DDIEEdPiSUsxkzTMas3UBVtdTE/Noc2gU29ogJ7WQZzJjSXjuPT1L8OhF4+jPksYihmWTU3RGZDrSzpRBAqlwUzP4yi6USKolA3i4DiF4aLI9sVR6Ith2fgAqpjHwuKsergMoDZ6xwzOQDrvGJmnxGu9hlatgVwhg+fv3QtMZpDL5Di6b0olmkIyjyDOR3uZGxmQU5FycUGzy9zArMN9y04kf6LfuV75KEXjSTSjLVzy5xfj2YePoTA4gw4WbUjFtW6k5qF6NIqp+Rr+/JM/ALJrECn2Iz++FsXSICo10i0bQpLbbI+xdFFj2IzePFCJjuEztq6szmVPOLgnty5coiJSBcBN4jDdtU3vZ0g4V2cu8s4T04mWmdQIh925tOUMHolqlItvQJ6a+LkEMVwqJL6zHNhMiLozWMTIk9dj5ye+iZ5fP6M0bbZdw57OLCbjHWz86/dhaPnZOOOq83D3N7aj2XQ2iWpSGynd6kPjLbMm40YyTSiL0kJK2bedm1OdSAofa7I6c9MuKZI1JNNpjeNR0VHAgUAvOy1JqjCSxjxWLt+FZHIRrWYUuQFOA+WRTGfUP83mehFNZJBO9yr7Y13IMRi6tFcX64ghjliGtWRELCe2ctKdBTQW66g1FlCj189iGeW5OTzy9Db85I57ZF7Nh3nhmWfhsgsGUWyvwmB0tdH+2Hohw0Ynbg9S/b2Ip3KIDHHjvhTP/OgZtUcOzG5GkJmS1jQRWva42dIbHH05BkqrcODRE5qMKZV6dA/lseRmUHkP58sV1KpNVBumQ3zixKRQ+J6+IkZGR9BpdhGViiUXgpOl5TnRNXcBtZpEYjGt4yRdHUSMoLyNjYAyZaSSf5tjXKxDmzU0W1W9ZrY/iUIpg9JwEYt1utVzGiqJeres0oIpIu1EQ2pDLwZ46vbnMZQeRoQqjqfRD2WiJu451TaJ6prtjQbVSUmNccyx4MYKTRObP5BKskWk0I1OsovL330pnvjVIQyt6CJIT9n6s/PMiSMAnWaI791wF25+YBJBbgSx/mXoXbNGrSt2MiSNxIyGpZqo2wTbDFOSzahcPKxzQ5SZ2YLkkZg2/ya7Zmke11tlcjNQVd3zkvnJhXKx9RM3JQZtZweoKBrQfyhktGVLKYZcYMPm/B0Spjkpw8hlBlDOe1cnfQTtP7gMy771Gex52ftQoNdqq4WZTh1PN6YwE29g0yc/jGUbLsbKS1fhl998TqmkSahyTtY2rPVBjXLJZj5JFFww4lG7vi3THqV+buHyz3wYhOHpm0OgiictR/AUDNhCaNYQTSSNjJEJcfErVmLjRSvQbLOma+PAzqOYmSrbYqi2kE1R7yiKsGISI2wruGdvi4Slgzxnjb8svnA0wCInVeJAIhUjrVW2KDz5Vm8cR74/jlvuuBVbH30c73zrJrTngebBBPoLg0orOxq/o0VKEem+HgSJNFKrchi79GXYcv2zmk+eaD6GVnDSdMUEfzHA0cN3A8654GXY9ZvDGgDoKZEKSjc9Iu3W+uKpu0jt5BA4Mb2ogMfxPhp0jwwPq1TyShNauM4ki382BcdT+timEMLRSJOo1dQPMRCJCLS1WHUSaR6Vvd6YNhb1t6xWZX/TCctziAANRBIN5IeyGH/JEJK9EWQzaWx7bCdmtkxLWYLXRsCS7cLFhXkro2j1kiDLy/qlTFs54pchcpzJ6DPJc8qpXcTjedWstVYL+WVZXPSWS/HgzduxfLwH0b6jStm9bKtknniX2028/69/gD3TRQT5fsRH1mBo9Rqx3yQWWG/pXspbOogiSnIJcxAe2Jovpv2qqZ3QOoeaYzLvZqr8y8IaJnYGOBnp1eRZ+IA9nN4JDWRgFKTjHFUfqFPbpfdMW4oTnF2MDfSojxjtzaEQTSI9U0P6yDzyQQyZ0Oh8nJYRYubSbTbc+3/+VUSWj2HqlZ9Eu07fmTbqQRf3Vo/gZLyOc173Rlz+rvdiYMMI7v72riUShyhyTppVrCanC8XZUpLjBbjJb9a0hfiBiWJyQc7PmbcP6WgLC2XUm019Dr4IEWcutlazo9bJ+o0rcOEr12Pn9p0oT7YR1uyz8D6xnrUpIPZR3KA2g0eap7YRWtjvkxwz+7BqrDMTIbhmmQNH+iIa/TObDNZiXMwiM3YB8owi2QbGNyzD6PIUtu16DJV9DfQ0ep1nr0V61qaF/l40IlEsu3gtCmeuxrM3PC/q4Ynm4+jEp0BCCjdmtVpXxJ+e6cNVV/8+nr99vzIgyu+QX8xgJuRW3NgoFqpVIcknpucwMXEC685YJy0yotAqExRALYAQPPNkeNaf/BmpX4hsQH0rcortz7JpbZtesNZFp6PhD9OHMoUSOfYRXHIqFaT8MSgzh0uojWYHB9dUPbKAtRcMoHdlEQ/+zz0oZcfUZ1YJ1+miTMlcotSSCWIJY4rTTJ954kZiEW1czUDnrBwR6huhxnGAMBrFqgvHsebyjbj/hucwtiqD9OgJE7d3Jy7/w4EI+m9d8bb/RCs9jGh+AMnlZ2B0fBUqi2VNSzUrJA41jeevxUv2FGm6DFIdySJHui1RfMlhR9vLP3UR/CK3WuCU1Afk0yrPQWkKS1ep00a920UlaGO2WUMtao6g6jG5FpDVwaxnzDE9xqFrJz/C18h0I0hH4lgWy6IYSyIZOFUL1obpOMa2/xQnvvsrdL95q8TXNHoWAPdWD+FgtIqRM8/FH//Dl5AYyuOB/96j9IqRh5uL1iCGIFvN42VkZeLklPK5eQhQsX7jKcs2kLxuKhW1fCq1hhBlL1zOh8yNhxTw2qsuw/TCNKYOLjDJVeZgGAAtNHgfTLGQIgIqDQJrpnMhSfxM8q4mvcLvg4GuZSNyGgM0QREbCm93kJdReFe1T1xjbUSYOYETWtssE2LVOT1Ysb4f9/74HqzIjZpCIqCZ6Gwhg0RPH0YuW43U6Bieuv5ZpHIJzGIrgtSihvQjEdaslvJue66B93z0A3jy5h1OEzpts8Ed6kIvuuujvUkTEycn8cKBg1i5YqUc8lhSeN66XxPcnDa4buqNavE6FwquBbLYGJj5/IxH3LTZU4eV6BmmUkpdGWDJ95ZAmsdV2I5r2SY2qVQ+AzMm1ymnLKmJVryG5WeMYt+2HcjHU8jSYocGZa0mUlQa0VohN7uDRq2KTIZa14biExPgNTAQcu1Qj4xkmVQui3YnwDmvX4++1Wvw4I+fx/CqNJKDxxCJkmtl+lpm1cryMYZXX/t9hJkCYoUR5FavR09pQCCdKaOw5SeKn+mVc+M252XIztOWtX/A8kLpLenGxD4I7gYIbi2sNQKGEdzEveTGSQdxVBp1nIw2MUPurWmfIqmFazrKS9QqH2nc3KoYGC4lJkZtNa21g3JNYFVhAL2kqEUjSF16NoZ/+E/YecF7UVqwi+XTboQdPFQ/jF1hGcNr1uOaf/4yOuk0nrzloBucj6lWJW1Pin6sq2NuAH1m1lJXV/96aRJ+wkq1opOWNR75rVTTr1IeRsyVhtQQudHGx1cglyfnloPzMRmDeWCNlpj8ko4SaXpk/lDGhkqGFDjPZMXSkayqZFFtgJs1HE87vo6EzCUI7mw2Q0OOBYRJQTIuphI/n5/AIkKpzglqaIV1XPGnL8Hdt9yJlclRbf54NonSYB/i2SLGXn0m2ukinrphO4r9GXQKL6IRmTUiP/2EZNbVwCN3H8Sn/uFzeOymbSLJcAHnC1nmfTpxzUY1wHylhv0HDyFTKKK/t+TorhD/WYEukXQaWoH0vCxAsGb0AweGigpEdKZfAozcZJml1bwvMZlUe4cBgWP8+SXdaYNdrP3H2VjzI+Z1erBK/K92oB5rM9bC8rF+zJ84jqBu4JQyApVPtJupoZDPaprLanCzRhFTjWoc7CqEXeTTBcxUaMaWxiV/fj7CRAFb7ziEvtUpBPn9CAPTuxaCrtMTuOmOh/Hft02ikyogPbgCpTVnIBZJSGmDa4EIcocEmnaIUqKMT73zYmr4c1uIl0ywkyi2tTg7CIRykx4bR/BTlypbBW99pHYsgulWAye7RBQ7iMaZf5skqRBChzKfcuezgWu/kUm+9kg0R/y0yZkO8KO5k3ptugcr0j1YdtPfIXbeRhy76MMA7SzYL2XWGQUerR3B0+0ZpHoG8Bf//m9IFHvx9O0HNMequpbNcg0RGMVNoEcyKVcCetMI/HLWi0x/+Vl403jaNSnG5cTOadZEA2NTKAReuvFcRWIbAneKjhyyd2OJGtVzXGcJBzBLIXc28JaTMQRqBcXkfMfIzmvU5FWbC8ycFzhL7IcvpGLoSAeLTu+Zi1kpu9LqhkYBqeIhPayQChJlXPGOjXjqV5tR7GaQySbQt2wZYqkcVl25AdVYBntvPwwkO8itnEGQqinCN+pmvcF0+ZYfPo5PfflvsPmGbTqJiEzLoiNus7tSWIwncOjYBKZn57Fs2YgWNFVPSLThBhKRIpdRqqzhCfnzWFamckQePmyFcTCCxAn2N40vzp4xNyazHdmZuhYjf1dOeU6CVTI2ak2ZionNDTEUOxkl9z4aLHAcAa/X3ApaGD9zGXZvfwb9qbTKGvZ3tWkLBQ0MMIMiw4knLj8D8QKtd7WDOFAQQQsxNLvAa95/GbY/fxRzuwMMrouind4nK1jvrMjnVq038fYP/ztmo+uVJqfHxjG4Yo0OPa4JAlKScquW8fl3vQwvG+uIO9Fg6h62lIFxuJ7bivxslQPEyEnw4b/dnFsZ8g9cSBwYrkZDrHvbZYitHdQbzE9NY37vFMon5zF/YgadahOpTgTRkG5trCtNbiTmoHBrHDGNNOULJsWqCEnlokwITYRZR4YBlmUKeN2ztyGaKeLkBR+20SaiZ4yo0QDPYhr3LRxGJJnDO772TQysW4Hf/uQFq6NkMs0hAecWHo8rdSNowt6t6k+mZE7xgBtcZPZWG1XJmjBOVKXcwE1o1Lw2zn3JBs3JaqyRtbEYLWZHYsMFjHiWuhC8oOuA5lCDCGoV61OK8x2Eiqqsr0j14wnPoELAwtd7YpS5YMATRUqHyaRc5zTepRSqo0XE01ejctTI4uxmvSYXt3pzFle+/Xzse2gbcok0hlau4NGLtW96KSqdBHbfcRCNbhXFNQuIpG3OlvIpqhEjcdzw7fvwqX/6NB67cQcyqYxOWzKcpCXVaGB+gQGti207d2F85SrVf2mmyOKoW/+fG3ChPCc9KA1exE1czqfEGoUk6OQ44/LHZb3veMT+AGC5Jj4yyQgajjd5UgUtAotyBDRPJrUc9Xwc0EYJHefP5AXhWOZ5FZZmt4GRtf2YOXEAyRqrQ9P/5qnL0pmBk319BlnOVpMwoqEHBV1rMTYaETTjIV7zwU14/O79qE5EkBo+iVr4InKFJOI06kqYYTlBrGs+9FN0C8sQ61mJwqp1KPYPihE4s7CAVq2CwSzw1Q+8DJn2CbTCONLxAMTAqVbC9hL9mdJZYggkpjBL4MFH87Ikgp8Ux2Xr2YgAx8MOfrZ4FN/83idVGPuWrRCuIDBt5GaI+vQiSqV+qSgsTM2ifGIOE3uOIqg1ETZa6Fa6CMj6cYbYUozgmzrDQyqusiJhsPzAoaeQ7EQxcf77VLtIwJORKBrBi9EKbp99Aa1YAtd88WtY/6rz8MD/7jRjKKKCBDlEljAgnqcAbzYfsCIaTwApVBhVkX+fmplCxGlmsd5imsxTPpVPo8h2Q3YQSal4nNa49yWA09vSInIOBamkqWtI3lSiZcY+4ukraRtOHXWMQM7711PgUD/5uMaE8WN9POW46TUiF1JQ3ZwHJCpXr5tmcYNlwYLb+AHm52dl07nxNWMI52dRjOQxtGI5EMthze9txGwZOHj/CTTDGlLLphGmKCzAUTe7H1y4P/nuw/joVz+BR37wHLLprMTuuIj5fjK5rlYxOTktOfO+npIR+cW+Ms1iZg9ybjxlNKH767+I5PpTV9pU5CzTKlTgH21gqExBNUdrvSnrYEYSjeh05vvwuTVqRH1NsZGDHiLfcPrKPVcOlXgvKNl0KA03l0cFOtbL7TY2vmIcL255Gj3JgvkIxRMS4FP/v9NRz93PQiel1mElEnu99VYMYT7Apr98Be65YReCZgyxZXPYvvMxDA33Yu2atejr71cZdPzkDP74Qz9CmCshXhxFduUqlPoHUG1UsTA7j8FYG9/4wIVIR2fQiUYws9jGkRNtPPfCIew6SKFCUugIUBpDgt2JFf0xrFpWwoYzhxH8b2FlGOuEeDxawS/a0+jEUvj7D1yNs84Y1QcR/Y8JO2+6G5aWiTQb4lT/Y9Rr2Ywsv2RMz0b7QhURDq9X6xqs539bE1Uszs5hbnIarVoXlU4d1z21RQPhBza8G3EaLsWJ3AV6/ZOJDn4+sxfzAbDp7R/BVe+7Gvf8cDuChlERefrZ3GzDjMbI8W22NIvJjXSUw/Ipeseamj0jMvu4JBdwfnZuYUFXTV7uyjUrUSxkEDZ52kQEtFGrin1SBhyCNVJb0KQGbTVa9j3q/AaBshPV2JmMo4+aMZgZejnfYKZ/i/NLUbkupcmOGv5kJ8kLlptdDnu06UxaPRiYFUVNG54tphSqlZp0hDmFM1s7ij+59jIs7JpC34oxBPE81r75fBw7UcPhRybRDpoorJpBM2Kc5obkYUkLTeOOG7fiw1/5OH53024BbMWegtQReR1MVXnSHzh4CIOlQQwMDGj2laCeKW+a9BAXt3yg6EecMraVBTcT5OM94ee0oGHEDKua+Lma+gt7zWqjuNaM/68X92Pq6Gei6w3bmMr2XOeDypVEavi+Xk6HAUW1sPrJZhxebi3g1VdehD1PbhZYyFQ5kTCROZUmEjKI6bkxW/MsQQFFiRwGzhjA+is34K4bdiEVTWLDVSW02mZETtYdA8Tc3Dweefx5fOE/70c30YPk4Cr0rlqHbD6DykIVuWgb33jfBszMTeF719+NPQu9aq12wizaLEVpGs5eD0k/ThPbm7tFKHbAdPq7uWXhb4MKHuLoFf1fIgE2jPfh/33kLeJZsk9IXS8lJBQN4/51Y2Q8+ZQGM/+P2ryrTXU4epYgU1pTcrFTQZFN96a0rchSIkXs9X/xWcQjOew+511IEYlNxkV2JwVsPt7FLdN7MB22sOrS1+Gd//Jp3PPD5xFWYyIPqL4Vq6QriF8mXS7FJLrMyMnWglQWnFUj02VOBFFqhbS+voE+jA70C43W4IAAD6tXKA2zxBJzJ6k3h2ZU5wJhb5btDqZ+THH9VI8GviWMZ20I9ZmdGsPC/KLSSvYbGeGloOioLkojvRgd0XOaPXMYvV4XGGfpvpFeOBNbq1ZQayziirechcb+eYyuWCVdzHV/eD4OHC3jhfuOotibRXr5CTSCOSG4YbuCarmG3r5+/OJHz+GDX/4YnvrJbqSTGfV8+/t7tQhZA56cncKhFw6jVOzVxpV3UoIgVsbKAVd+SPliadzRgpa8kJxgAfWrubl438yDmcGTQw8mSqBa2pVs2szOo9dcDttLhtu+zcTPLyqg0mMius490p2cDBjKxpzDngJMB1iszGGhMY+RoRCxWhcl9q2jduJ6mx1mEjIoo6+U27wMVJVGC2tfsQ6j563GPT/ei77eHoxdyL40Mw5qaidVcbc7EXz2S9/Bnb+bRJAZQmpsLfpXr5a4QHl6Du96wzjuuv1BHCxn0Y2aQAFT4EjUAoyoyQogRiVW1yEeQ8vZzqj99vO3vCn89+eewo7j80rReBrl48D/fu1TeohEUHliGY2R1WsEMTaDCc5EEppEKRX7kMwWjAXDiEqLCykXmJWJ0haCD+VF1Si84fVmFfFOB+e94VrEC33Y8ooPYHCyKlS7oxqpjXoigt/MvIiDYRmRvlH8zU3fxaN37kdnhhs3q7qT18wNzEXGB+4XjG/60+OGpywXDq+BYmDsPVebNSxbtgzFTEapsbxz2GoQsOK4yi6VVapKPqAUEu305P2gYiSV+WUKzjS909aG5EnFfpxqJKVwfsvMAAAgAElEQVTKrI8M9eSC6usr6d+46dRycEPTTN0ZeIiHCGGNxnTikTcrEQMnN0N63uz0jPF/K2VUqwvoWxdivNCLlWPr0GjGsOHai7H3wBwOPjqJUl8BtdwOpPIEQIDjR19AMplFqbcPv7hxBz78T5/Alpt3S962r6+oUUWO2c3Oz2F6fgZ9mX7kZE+yqDqcGQ1TN1E8eZKRZeXacX4+l6k4B+D5JZKFPIGdSbmb9eZn5Hog44nsNAZ31k/MMigqV6FwvVJjk9S1DWwAoszSvIWN3OxscwuHSNsJr00t72DLykh4oAZ1uTaH3qE4Tp7YjfHSiNJ/b5rOZ8uSRbJBZLWlqVNNSZsUFisVXPS2lyNa6MFjtx9E32ABwxvYozdRP1qqRoOkyspL3/ghLGIUieIo0ivWo3/VcnSbLRw7dAzh3CS6kSwiKQZz1sSWLfjxQ3M7sC9t0qXx19O+9+SN/xA+u/sgvvQfN1qNyRQ4AvzL59+PsZF+pAsFFOJ59GRzZq4cJOTnU919GIdvfRCpiRpirQCtiOkwsb4sNQIxbyS33WijFQvQoWp9xB6wTheO/kWjWP21jyJ5yfk4/NX/Ree/7kSE/jsBeZ6U34/hifljeCKYwUK1jU/98LtYrBWw73FaH9KuMo4ux8SoPEH5DzfMwM3Hv1MqlL0dyqUeP35cWkp8XYqDnH/ReZg/OYtChu0Mi+pSqHT1r2aTVSdZFjE3M6eNwpPGo5r8fjLJ09xmWEn898ytdov9R6NecjOSyUWQSX1OCagTOeSMqtV2xTz9hLpakETfuUm0gBIJnezeHlM9c0m+kjwxoxp0anYSzdgMXnXRWiwfWodqLcC5116MFw7NYebZBhKpCCZaD6MRziLoUG2pKetIBtX7f3kIH/rKJ7D5+q1IJTMYGh5AEJBAwpS4hrnZOfQVS0of5QoQYzCxe5FOmqQvN2ahmNMCkwome+y8p3QUiMdxgvO32gQcmrd/Y4uJwZZf1WrD8AgOs0fNq1g9cGk2n6I18Lmq3ylmElvipmjilTL9/LU5Kphel1h97FKwd85yo96U6+B8eRapUh25bheD2Z6l8sXPpMtrKZV0puP2XNkfvuKDV2L7jhkc3VHFslVFFFfPL302ri/yJCqtNl53zXUI08uRLC1HenwdSsOD6MxXsHPLVh0SsVQKMRcUlBI7PTYBul7uibO87A67coT1uqE51FW+6R/Dcq2Nj3/x69i06Qq87hWvxJrly5GqVTBz12/R2XscwZEpxJpdpCi3QhSWi0+9XIs0GrbvGOLpawJC2CJekwni9GHZ/mAkdjsXrW4bfVdegIF/+yxm7n8alQ98E22ieNTNZV4Ti+JAYx6/qh9CtQO89Qt/g/WbXosHfkiyAN+fpxJnNbnIynr4WuBy3DOJU/XhOmactFgpi0zx2t+7HJP7J5Gk8zd5xHSrkw2Iobka5eNwPRFOESVSSCVSJiymuo0zoQlDJWWBZLeTI4/8HUb/VDxp876UanGtEm8JyZ+VxpLukVH95mZmxDUmsslTtJAvGFgjw+cKkjJutv6lpYddCdNxU8zMTmO+OoU3v/4s9OeXoRWmsOGtl2D7zuNoHiZzDJio349uZEFpNgXIZ6Ym0Vfsx7anQ3zkKx/DIz96HoVsAcViFvk8gbEK9u55EaPLxjTN4wVEeL3SOdYEmPlIibXGvr3bbAqCTO2oXhE3v+AKaZMLiwqyslrRYL4NgdBPyRuGcXKKtaz6x+Q+M/X1/V63WW3w3U5gm5F2rbTTZIWZcUpUPWrcaG56Pj9+n6c7sYaZxTm0g2M4a3Q5MtGERu24ljzST2tSormsm0mznCrP4M2f+n384odb0F8cw9gZeXSyRzA5OYnJySnN15JnX2kA//i9R4H0CFL9K5EfPwO53iKObtuBxfl5pDJZxPjaMbo7OuNylRqm3qHzVlguZQad5KvLArXOeAo/f/t/hfmFNo7evwOTjzyDnmpHOsasW+Pqldqu91/EakwEnQLddnr6qQU+XG1cZy/CyMeWiixCNNnvcngLGvLabfVlcdbm76M9V8exqz5F2yGdtCzW20GI2XYdty7sxWzYwblvvApv+ZtP4/4f7bGBfuk/2QynGTTb4uHDZGvIs3EYwVmbd+MhNr35Amx9bCtKyX6zX6Qwmh6ODczzpDaFhLZR5UQggNo+PDG4qZge2khigGTKPVi1vgL1K0ny4O9wMUpkrWvADVM+LjKBTmxZKTW3jVivlDWr2kO+cSajFoiGxqVKccrSlEHSt4p4ijOVnjx5Agu1Gfz+G85BX2EE7SCNDW+5BFuePojudBKpeAwTzQfR7syZ92+jiXa9hhNHT2B+cgU+9o8fxb0/eAY9uQIy2Tj6+3oxMzuFWpmqjD3i+VqWxNPALCK1gLgpnCkVsw1D7g3x5896XjI/L0sE/js3r8Tb2PtlnSy/J1L6rBzj4mdgYGqr9hDnp52ihaW/RkYwn1pj6p1Od9XoJkkuRK3dz3gxRBJYTIaojmarjonpaVTbR9Gfi2Mk14NcIS91EqWstGXp7dW1skzgfHRQiuHyt70Kt3zndxgeGcNseyd+fuf1uPbaa5BMGn2SG/fhJ3bhB3fsR5AdRrJvBXI8cfuK2PrAQ0hn8qIFxxm4nfSP8AExv8wzyXVWrWRz3AdN5y0N1AQIHlp1WZgkYOEGdXkTk2SdRLqId4EW2xrgrKZXdDTNV40guRpQObgWIAegqV/rHP9MCnhJZ0onhtNf9qNK0WQC4w//B7rFAg5d/GEEtRYiBKjULgpQ6TRx59w+7A9rSA8N47M3/w8e+vkBdMuExTrIpvPaELIldBuDCLMhyTz1SGvsoN6u4aLXbMTBgweR7GTRqlcx0DfgVAbsQXHD+tqYf+fD4BfbD+w/q+6MUxzNUE2zrjSyvEYB6ffSqIs5RcoaU0WemN5xQMCDQ1RFPCM6TUmcRgP5bGZpookbeHzlSszNz6NDcoK4z+bB68GgmdkZG/RutzEzexLHThzDa16xEr25AQSJPM7+o4vw9O8OojObRC4dwzR+R9MPMdPKtQoa1TIWZhZw9IUiPvqlj+K+7z+JTCqHwaEeCabv3LsDq8fWIJUxQQKhuKSvpsxFnkGRQUci4uTyOkM4s/uwnrfpGlvQl8xrta6NwI0oUy4OprSYXvJpm9IF00ZmQCwzCGRqXWqEzwKcHywxhpJRHHkP/DXye2rPxR05hKi8K884LskMi1KxxEOIjs9WJ1DvnsBLhlcoaKaiCdXjXNK5QlG6VBymCNoRrL3yLORXDOPuG59D/8AIUkMHUGnPqvPAykrOjc06/vP6B/HYvgCR/DIkB1eiZ+U4svE4tj3xGHLFfs1gRwisatzTmQIwXXakFTk9SkbJdL90ODrZGpvkiyB4bOSCkLmzmQrZEc1tlzDW4lIU5QtJ7cJtUJv4M5sRRUSZe7kBYPVs7YubnI10bmhX3ToFgq7QaS7ske99FomLN+C5V38C2dmKgCARyAhUBQEemj+A59pzIof87a034unHJtE8mUWM9Q0nPNwQv1BhN963JGcTUrWxgqF1vQou8WYcsUQMhVxRtZTUPdyDZxTnBuHn5GmXSZPGZ20HnsBcOPwfr5kbyMQHyCWmf2qIYq6gHrMWdYcSLaS3LeqGciaYwUS9RYeAsg/LB2MuCHZ3fCosAbFuF7lMdqm9UXdzmyZqXlcdTDS2Vq9gfn4ar9y0GrlkEalsEev/6ELcf9cOYD6K5csHMRt5TlRJ8bbpbM/yodXBw/dO4+Of+wgevWkr0tmsfIlypTw2P/woXnLWOTZQTkIGTzFxj01xUKqMGiC36yZQaIi6Dbir1SNPZDt5xc12JwzLCdbTzBjUI03EBdBQmpWL0p/U8qJyLR1OMhmvm5vEXlM4iAsMzIJ4TRL386m8a2fa9BjUGzUKp1F8mTpPLUwjPdBBs3wCq3IjKknYseDPkPvNjIKOgCQcXfiXl+PI4TpeeGoSgyPDSI3slN4VT3c+V5VkzTr+4Tu/xY5JttPHkBhZjaHxlTiwbZumzRKZvKi2HDf0paWBbJY58rqYbfK+MEX3AVL9ZMe00+bVxnUnqMwTnAh1zGECPpIpHQmApEvd/MZUX46ImtIka6X4o15725v8OtaPT1/VdHepTPHj16D3L6/Gts9/F4W7n0eXyvOsYUTyCrG9MY2HascxG9bw0W99DdnhM7HjgSmZaVGs267B6hx+eN+096lvmKhj1dljqJ0gV5XSownzi2kwdbWRRQYWTaqIZ20ax5qPlCg4QRHbSOpZaqInKU4t68eeYo/olLJecWimVQx2Shjrpu5SLlNL5KkwMNinf7f3si//Hj7VXJxbRG9vr4CoQr6oIGR1HeVW6vqsrKXn5iawfl0By0dWIJZM49xrL8evbtmCYtCL/sEcFuO7KBJqI4bMJIjyV6t4+qkG/vBPr8azv96rdlCuJ4XesSzKxznwbm00qmbw3iiu63rtWZMRZpkJkXOr9atUzHQlk2rVGlH0viUQTlM6uieGMHswi5mMSpKWnaDKdCRiYJuXmAC/L0UMJ2jnUWX9V2xdu9c61V0KTZEEn0pzuoeKJJo4Yg8dXTHDphYn0QgP4yVDa5FLc+M6JJktwgQ7FnU0unW86TN/godu24OgkcHAaAnl+GOg7JJlXJZddFpVvO+6X6OaGEaydwXSy9aif2wUzz26Gf39A4ilMzppSSM1BQ4DvtgO4p89ocjfJ9IiPdXWmGGGnAdPLXu5Nq5OR9cz0kZw43Kn6lc7Rf3MrmDqUwerEFWfFnkyOVNE9TCdnIyG6ZneiN1k9R7TreKmjcj/5ycROVHBsT/4AkJasLuJGb7FyXYVt1b2Y7pbwUVv/j38+Ze+hF9/5xmErUByI0yrPEe1WOxR6snWij5kpIWL3nQODj5xDFE6kDurTJlTq/fLn+NpYO0ev1i5wRURXUnAFJjvIzUIjgemMzqdqVRhgZ8zk9YaUW2mE9k+nxHajVRB8gY3Ir9IuvCBj3PK3gyNi8UrU87NzGsUkWljJpMTpdOfSLZgu1goL2B6agIjQ1Gcf94GsZxecu2luPWm32Esvxz5YgTl+A50A+uVtrvUvapJA2pudhg9A8OYeHoGgwMDiOW7mJo9ieH8iGpQa8cwZbU2CVNWzchKLN1ojRokQFSsLvV/GVzabXMSiNiEFH+ezCWjjSY1tOExDwZHsqT4M5TvUYeAmAB72q5V5x3rBcy5AOrTaB0QmtKyUkQIshsEIW1QCDixBtrKMP0mv5oYAi06W00szM1gsvEiBrIJrBkYk2WNTjzO7VIzLR7H0IYhnP36C/Gr729Fqbcf/aM0VntCdS1benJdTGYwNXkC7/z8LxHmRhHvW47U8DgGR0ew9+ktKJJVxdOWjgsJTiNZhsD70GyTi2ClGfeSZwNKtsdbazqXS2WBW0Zfru3nj2058vEGOt1jc9WzNFoTREsypwR1bMSItYw0hAnXMy93spsEUsRNdv0ouRfoxvP/XQ+Q85lDJYze9w2kEgXsuewjoNUwwS+pOyBEA13cuLALk62qdJW/evdtuOfGPYg1yAv2UyVRpV48OUVamFtEtVvDm655FZ7Z/DyyyQwSbLS7E5k3SQU/f96JbJvyhbsXztBMCh1CJCmYVkY2m1MN6GsPDVArG7EbzM0t7eC2qX7wgVYWFxS1uWFtEZtIGiO737iq37xxmrtGKlTy/fj6DAILi1Wl3BxlPAWQUctpUdTHZHoeF23YgG4kjvPfuQn3/HwHBhJ9SOYC1DI7EEQoisfAydqwpfo5VTgXEweraB/rCkAZ3zCKY7snZNZlz6qjU4drgggwA5ykZyjy5nji0jB2QxzS+2Lv2g0fcMSEr8O61Zip1ttmj8bqO9akBgoKdCJgSe4320cJ07TW4LjqbFNT4cv4UT/7Hadppjcw6SANqstnmA4JnB5qOjM3Xrcx1BjcqTDZqDYwsXAUtfpRnLtmDfIpuiPwVEyimMuJQHTRuzYhjKVx1w1bsWzlOIL8EYTJSUQidr3iTXfaqHUDvOPTP0OQG0V0YBWKo+OIxUPMHJlAtm9AnRKbCIuKjimchLRWlWI2fMLRWj9wov3oWGgCsPT5Q9u4OgUdxO6lXsTY0H0I0abDPJFibl9fx0qmxrjBegAauHYCc6KuWWSkNaSLDEsnNL+/1CDniVssYPj2L6PS3499V30GqUqVk6+ajOjwwXY7uG1+L17sVNCMRPD3v7wJB7eHWDjYRk0Cb4YOU+jLZESZZDfwmj96FZ5/8lnkUgVNuzC4MLDwRlMwTSi0Nok9SC4e2o1ysRoZg4CKtSxIOuDgtcUt6znqlHdTLp7mp15mtQYuWHF9azWUeou6LvNqtTaG94IxQTbz1zVAoiPbDn5fPWNJqhiyXK/ZCKM15SOYm5s1KZhqBXPzM0gXFnHROeeh1uri5X/1Wtxx/e+wvGc50sUoKqltQMC+qaWq/Awc6B5ddwmeu/8wEtU8xjcOi0dbjPcYi8xbmDoqIe8zUXXSGvllFi0R3SNeL+WKfHvLVD5Dsxh13GbrRds9NwsWnqyUJDWgy6fdIrQwhXTaX+rLcrTSrRsCWkJYnTqkP5F4Xww45FqgTWdCyhFiWAmLYW+ZiLQJA+rnKB7XbGChXMbxyd1Yt6KEUjov76BcOidKJLOnTR+8Ant3nMSR58soUGu57wDaUng0NVQBYN0Odh+exRf+7QEE+VVIja5DaflqzE8fRqvaRLK3T9x5dll4/WQJ+iBH4pP65Kdlrr7T4Q9WtsqUHfP/nhq6QN5BYn84Lx+lYFKlt5tHaqLsIW0f6xdtusMI/qK2ufpORTSTNd93cv64Ek/jQ1JUMSKXAAYytXqyCN5xBXIf/DPsfc9XUdx2GKGrMcmkYozZPHsAT3RnpSzwse/+C7qFVdj36DxadfJjCSjZbCW/WLtcfNV52LF1J0ppRx7QWCEDvfWa2QKyFMsQZY+amqAYh7TrOiWLhaJtNvn/2KnK00AGWg0j2osUQMnXuBFBuCEqi1W1pPjgyfbhIjVE0NXMsjqpqHfL7wlkIpHekTG42LgZ/ICBwJ66aSHz9/h9gl8kQ1TrLczNTyGZncJF55yPVL6Is992Ee67/jkMl4aRzHTRzO9Bs0WXObsGRvf52VksO3MTnr3jKMbPXIG+oTwWDswikcqphSTwx1ExfW+T/GTW1MwseLKxx8375a1rFNYc51jZBck61YrWjW1cG7D3X6o36zZIUOrrXQpexAHIIdYGVWpLsoXJmfrSTkir62Dw2fN+SczeqbcYW40kDL+5DCBV8NagekcbmVRcDrdPTB7DzPx2XHDG2eZkkM4hmc0iSAa4/L2vxYO3bUdnIY7ScB/i/XvQCo07zo3rg/h/3nAXHtnZRrJnLaJDKzGy9gzs2vI4Sn0DiBd7FdxYz6ssEOEkpj5zwDlhmejBJta4R5bISjbUwnvpeRLBs6MXS3PK+wL5h8WXMHBF4PFSrcdvmK6ytoHzZ/HppRG0pUFMdUd56FqqpBNWEx2urcSGrUuXooko4meMYeDGr+DQz+9D4ut3oJUIbIiBvOVOB3vrM7i9ekA3+8Lfex2u/tsv4tH/3S+QhuR/EgsicdMzHjt7EEi2ML+/hnQuiUTEGFGGk9tMsdExzUTZQ+/sH9oYmRHjGQykc+TYTdrwrs3AB6bo6NJkntr8nAQ7uJDJhBK7hxGeSn6uByn5W6dgz3tNEoI3txapg7alAmH48MwHlq9LCmCrzkDH8bgWFhgcSPbnMECljoXyLMLISVx27gYUV4xi3ZvPxYPXb0OpNIBkpoV6ajc6odHzOBjBz0qlzNVnvxI//taD+PQ/vxeP/fQpFLI9qv3ls+PS/6UA59M0qydO8YOd+L0tNmOK8TPa6Wajn7z3XKD2/Lk2DMziZzMlDVsjptNt5RWvT1iHq/kM1OrqdbSAtTh58jeEa7B0s3LNnrMnZ3AjLAGObhSQPyHMgddIZYw2Qb46dh17DGsGSljZN4I412U8jdKaEi6+9hX45fe3Ih6hYF0PUNqNbruu4Rpz0ON67uJjf38zjpSTiBVWITG6BqvOWItdW55BaXgUAZlj5D+TlEIEmZvVMdKoeWYgccRQf5YFEac9zcNL/043DGJGAYKtIy8/JRbnTkneoBhrU4cE+5NCD1CkDIuYlmqae7g2tJN1JaTO2VprfViPkzef56wHVlg42AO1Af1EXwH9d/8rYtUu9r/hsyJ3sNdFyUve3JNhHbfM7kaVs4p9efzDnXfgwR/uQyZOXWVyUFvSpx1Y04uB0T6UJ+jDQqmUMvpKTP0c2OSmLeQzG7MmPReMQCWJiiVMnFojfM7KwguZuRPaVB1MTpWDF9x81BAyj1x7KP4UlxCBQ1k96YLXKxYPJYGc5QZrMVIifbrnF52eBetxPtBGS71QlgIsU7jJJyYmQLdDMoGmZvfglReci8L4CFZdcQ6e/PmLSNIwLdtGK/8iELAt09CDF4BDe8vsejzyqx141yf+EIc2T6gVR0BJ7BwnfSt0XsMbVOPIngZOmVay6XrZXK5lJ1zEhj1QRJ1fKgeEbVjqyr1FUIe/w03ja2Kesja/a6kjnw0BJVtHlk57tVCmzEKl5QYRA0XTddqTwdRsCzzk/WdQNVzFVFGMJmm5BK9loWxgGjf/8YXDSKcmsKa4BslsHKl4GmsvW491l2/EL777FDLZHEbGc6im9iDomqyqyeoyECziff/vFiyiB/He1YgNr5SiSKNcQaanF4l8QTRfL+fLtNnPWBN38Iw9May5lxzeYofOqUCnTb997NLQI1hEkj2rxxMqfCrp20I+yWFEYP/Nn2AOebBI1zUtYf2buzn8M8EQf9RbAmyRkUyeZUNDKP73p9A5ay12XPIh9FIbi0U8a0m2Gbot3HJyO04kO2iGdVx35x3Y8tAMwlmDzaS4H1vExks3YOaFGW0ioqZ8h9mZOZHmrTfm1SttzMu3I5jSSjZGd8gWmAm5mXyNMgbWbY5AwpuptFgqDVTEJ7BlWQi/eLIYD5kLlUHBojK9l7hYRNhfLKNUooyrnTys93p6Tuk6GzvLakL+TmWBKbLZiPhajekjpT752oeOPIerLtuIgTNXYPDiM/H4z3Yimy0gmW6gUzygul896oap53O079jJDI7snsc7Png1jj1xEulE2gUfA4P4VXWeQAwUlm055wtHDmDQ4joxYNBOTKs7Wb9aNqa6XrO1liG1HEXW+MWnnChIwOCz86eu3/Q8xetSyLDX8/8u7W6Bgk0paSylx9y8TlGS18UAGYtSY8oZRPOaXI3M+tK7O87MzePw7G9x9tBq9PYwkMbwpvf+HubbIZ781SH0DBWR7VtELXEMQViXtKwtGTLaGnj3Z3+GTqIfmcEzkBpbjemTxyTQx42bLPTYmJ6mfeLamL43K4MMch1cGaOSSlrShgdImCAwfWUNmm4feXl4qgi2qGSwtJvGcI1fqyu4QSxD0Wnj+r4Wu2yEzVpJdkrwxrHuM3DAjntLdwzU8GNUZGkN5IqIXv1ypD77V3juqk9gYLYhoriiI1sp3TYemD+AbcECupEQH/vRf6CDFTi0mT24kKIPeOklG/Di9gNIMd0KIwpCSkXCrto+kuVUe6PtLCdYn51Sm2AarDE0pb8eLLJUyNfmekpMs2ocjK8jX+BgudrmOn0NYQzQdhGfC4r3lAuaG5lUQ6tPTdJUJ4joeSbnygejf6OKQpVStTZULgvGtg3b8/e5IaSEz5Oi3cRiuY6F1hQuPWcIoy9Zhb7z1+PBm55BqYeDIh20Mnul9MCNR++g2mIFYTSFp5+aR7cM/NVn340dv9wlIkgu16P+NEE5kd4J7DEIOuKCyY8aCczKB/PbVe1GkobQ0oQGJnhSW2sLyOcKCmJ+Tla0x2x2qe+qk9hZ3XCteBMyOw1t8ovvytdMJ1Ogq55mmsnQ4sL3eINM2hg0TJOYJ7G3pzz9JNe6dVkin5ECcbWGQyc4mzyPlcOj4pxf/fE/wjNPHcXUoSb6B/oRG3oRYZScddbTxuASyFWp4z1fvBVBuojU0FmIJtNoR0IkMr3I9BQRTWfVnvHlmW1BZnYxE6B3Na31cO3z0J/JU3gpV2RYTATB7uWX+oPP0juS8qWImHNop+kpaac7cEWuB/Jk9U71tnT5u+rziQHiCnZaUbqJGp+WKgR4UEi1TQulbB4Lg1mM3fFvOPqVH6N962bz/KHyA8fx2i1sb81gc3NC0z1v/9cvYtXZr8JTP9uNdG8O6zesxuG9R3RTmIYnY0nN2JpfkW0QpkJyqKcJssbkLKAs8V4dWd1HdC4kXic3I3/HpFMa0olmmqcb7ni7ipCyhHSDCm5I3BQdrNerqB9ACLWsP93pLlTcUdx4GlEgTf1TaguTsU7pVf5OpS7wRWkfn4mUIpjutTA5PY9KdwEbz85j/CVrUdpwBn57yzbRGAv9ATrZF0z+1WlwVRfLCCNpPPrQBAYjWfzF378HT962HYl2QmqDYtPBTMD0rH0dq7TwNGacJqtaUr3wih0e+VTG0ek4i1XTRPZZhA+ACvSOJWSKkdbz5QnDTMfzc8mqUkakn3X2ma6OVr+eo6ZsIaq9ZKi9rlsaxca29wFTAcBlVabfXHNGajT/aqNaKWP/0d/h7BXLtH7e+sV34J5btiMV6UWxlEe3j8bW1F2O65mS+cZW4ez0At77d79AkMoimh1BrVHD0Mq1CHL9SHL6i1hL0vAWyxhs4yqbFe/aqJ3iO2jzdtGVbI2RMyRpIWvbLoLdY5cuORn4Rrnl7ZYGKyWkgqH3u3WbTm+oOsZACD4AzTA6cXR/QT5NUprqWiEmoO5qHd5URaEIYqU8Vt77bcw8sBUL190g7VsnbSTPmqPtMn5T2Y9y0MAbP/8hXHTlH+PuG7biyqs2Yd+Oo4iFEGXN4Hb2vCgVyjYCwR5OACUNBVwTb3QAACAASURBVBZTxdIbayNxkTjK2WnUQxMbM7IIPyNBEYmOU2vKjZx5fWhFezkeGEBC4gnvp05HTcLUMDg46OZ5rffosQJmAn7OV/e7YsLs2iDRmJ2ynHBp2YCBmDSRuGprkvZJAaSlRbnTwDkX5TA2MorSmWvwwM1bMTI0hHiuhjB3wG1cowmWFxYQRpJ46MHjOCM1inM2rcUZl16EF+7ag3KVxmj0ETIFCGPu0GjMaXA5Wqef3OF9phm2v07dM4chMHiaLA3rSjs9fGlgizO0ckjgyylfKqt5rT/MZ8ef4wZRf5ZC7sQiWM5wnJJ9Y4KhyugMe/FglzGv7NDxPV8/oWROF6HOH95v/l0Cdd0AR6cOIhudwdr1q3HFe9+Au36yE+lEHoWBJBKDvJfMTo3h5dtRB4+dxMe/fCei6TTiCTouVDEyfi6ifSMIqJsdT0i3mffJNqsRaLS33OGydDg60wD1fV1m1glNxlbFyu6xy2Wz6dnvYgG5WGARsKPepi0kk8Rc2pRehoQbXBMc5tInbWZPtnDRWUgjZTzZ4nBK9fwzazOeIkTQSvkChh7/Dqo7j2L2A9+0XJ7TKIyW7Q5muw3cVjuAxW4LL33HlXjt296HwexyPP6bXcgQhEmZUJdno4gho+a81Q6iw7m6kbWrXvi0TIJPXOkfb5T7XZIguEDYtuFDVt+NKQvTadce0qLUInR1BFt6ra5TyDCghikh081Oq24kFeatdFuv17UI1cAX5c9SS2YHZIEpqGh6hsCSSZuK/OECDBdQo9bA/OIC5soLuOLtG5GLhYiWhvDQT7diZNkoIqmT6KYOgw9eny/oyn40CJJ45rlpjAcrkUkmcOk1mxBms3jx1xOoo4pItItEGENIdQZZUHYQ7TozNUdL1MZjuuwGMvQZ2i2d1Nqg/kQ5je2kZ+ACuQKRo/rZgeG7ECxvjEHlBc2ZLtsYnAn4i4rqxAmWxvHcbDXXH19bBA43G670O8ZAaJJA3PAyg2sYgYanJw8RBt7JqWk8u+VuXPO+N+NlV7wcD/3sRbHC+saSqESft1ljR6Tgg2SgOnhsGp/8+p2IxTOI0Y4iFkHvygsR7+1Hh7PeZJLRtJxZmKWd+nzClVygs31oJ7F2JX/PeVOxzcl1J/R+z/JNp/IehxT7COVTItZporsJ6fPo8almsaKc4wsL0nZv6us3f4PVMA/ow5IU/Ywb2G5uG41uB8v7B1H4zT+hOVPD8WuvWxq3s/QOmGvV8IvafsxHWlh79cV4+0f/HlsfPILeZC+iEfbHDAkXgun6tdLn9Wn5Eo/YWhbyQfVyK6fxcDWvyeEAmkUXC0Zsd+LmYgZpUsoCgp/g8Owp3h+ioNXFiphRsiBh+8MRDKhW71Nj3ikuLO5BSqVaimj1Ne+3MaYog2qRWSqJAjSkD+vaSkTTG3rwi9VFnPfmcWRyUcxMtbHv8RMoDZQQpI6jGewz+F5JGXv0BDwCHDpYRW9lVMBNN9HBS990HgrLVmD3nftQmaUaYwJBzJU/zLAoYObKAx+whNTyfy7NzWSy+oy8h3SC8Pffja1YUD+dyHPa9JEvT5ip0AicbTCF09N+3nAS27Qee+Az47NgENSn5HpUIHTDIW6V83eNd22ZlhFvDPlWQHTWNvze0SOHMHxOGhe87gI8eOMOFHvyyA9XUYnss9aNzMpPHWS79h3DF75zP0BdKOIRuRzSw+chmu9FLEcNK27cuJzo6VniuQMKVk7myPxxA6XiKpe6xlPQHtAZbZs02Ltik1JlS1+WNrr+7ml9HjRQu8RB9aYaYVQvnzb7B8oTwvpN1nc6PV3236N8DE9Gr1xB1Hi4p4TBn34JtVQKU396HQLnym01UxQLrTpuLb+AmWQHF7/3arzkgj9A7UhWxHBq/LKSsVSsi2w2s+Rw5pFkf6O4WQmc8Ob4z6h0x/VVGY2LPTxhnU6wd2Vwo2QUaGMqafPHlkZazQTnWdRFf4lD8fYeZOH4E4DyJYywBvQYuYDXayoQnSWKHj+Hpm3o+sBUVSvXUmV+JZKkQrpB8m6AVDaDcrWMNVeNIozWcHxXGQefPYGh0UGEycPoRg6Ic8yNG+XIZtxE7SrTDVSOlBCPZZCkbUw2i9zqJM561UaUJ5vYvfkFBLWkVBl4DU2q7bsMw0zHHNWz01TdLz8mV9fq+p1mlB9/VOotewNPBNE2toXp5I7swCBK7Vp47nek6OgIPD4dt/64pY+MSQQM1cryPyuk36RX/X23zLGzJAdE8I3BVm1Luhh4NhuDcHYCG1+zEfddvwOFQgaF5VMod4/rkjWwIA65qaLs2HUU1/33g269A6WBMcQH1iOe70OHBtmprH6Hp2087daAH+tzhgOWevvDkWm8gZW6fxF/KAUIdoxcIuaUb9N4YMZQ5FPyofqg3KRuQkhC4K5G8RtXN9ydCL6INgc964fyQ/ovgjq8UaoJw1Ath95SCX3f/gSCdatw6PWfQqJtg/F6qEGA2UYZdy7sx/FUA+/73jcwfzyHZKtHahFcxAQZ1Bvk7zj4W5HX1ee8Po/kMoAwHVUEdEZT3pKT12u1sVHiuDgZufV9iZbbtBDracmKhAQ+TDyOBHUDUMzvxdIxN2rlepCkDfL7cQq7OxE73gu2pHif/KSJ+qcUQFetHrd5VV13c0kAT2qN7GV3A9TbC3jZn23Ai3v2oXqiiYkd82KlxQv7EUanjLhAxDcWaEiC6d7ciSlM76Xsar/xp1NZoy4mA/Ss6sP4xmUaQ6vXotj71CFUjs8h3o4DHZ6yvCd8RubiTqoFRQAJDPr6mOORzA70HGCnndYDw6ysVt2mk8gawSwG3axlE8qcLEngNYl+q6EGYytJh15kC1fDKkMhU6umZ677tZRJOdE5x5MXJuH48nwdM9kOsFit6NSWiigNrocyGDozhvv/bxcGh5ch0ks3yZrxn0m66YZuVrqNJ57Zj2/c9Fs0W1QETSJJadaBM5EoDSOeTCGayiKgeXgyBRYtTIE9wYbrm2uB18z+tIIz1w4F4pzwvxqSrssS7FnOGveUIJXfuKf/ly/CByFUWObXRqZYSkmcRrD6jS414c3kw6JQuPp6px/nLsbyPZQSqY61xTn89Q8iuPRlOPSGTyPXcmOCtO9otzCPJu6c34/Fnjiuu/NWbL5jL9JBj5QCeSOVUrgeIk2lWYP495WcqNNdVr2rVMren5uQ+lS+Ac5/07ifs+10B4K1Kpwxt5HuKXQW00A235ug1RKoFNhp7TeiT8WkHsJ6qlrR0IOXOl0qRVyNaKdGIIEzWb6I9GLfU3bkUkeiokRUCfxU81Vc/ofnY+fWgyjPVjC9awGZQgrJ3n0IIxxMMPUInrj5Ql4LfG5qAhM7ExjsWa9NyAkXm0VmfzSObjxALBVBcVUay8Z7kRjoRTpGzKOL6gJQmamgXWmhVWmjQqvQch1RyuxSmYQ92UxS/GaVMV0GNNNCZl0rE2s6CHAZkxK5pPllLTC/vvg81CEQJ4A1vu+XG+XWgoIBTHxG9P7VkL7zHGJ/l7PAqqdVG1Nvm1NLTlCO+obuvdXB4KQPSxwy/XozOOOSHvzmxi1YPj6Cbv556VJbu8okYw0TCbHrxZO47tu/QbPTFc85nutBduBshNmSAKsY0WZiAWSmxVNyP/AYAWEufg5+ziWlGAES1t9VOeJKFB1Ep29cf8r6k3aJLOFOTZNYNZ4rbxiNlJiqqLZxTCtLfE7l3F7027+mpQJ2CsoYiZQzUgMYvQCs+fjbkH7/n+C3V30UK8qGVMvXp93GRFjFXdVDaPQk8LXN92Pzz3ehlB50DB1rm0jIu1wG9YJ8veOjrrSgXL1gLQMzxubm42fSxpbVg33JOtJ5lRrybKm/r1dVL8m825zn/eSKofM8BZymFJlEro9NYopNv3A4gGbOXMhOtYH9YpeeG2pJdNrECHTiO/oogyhPNqZ3XOy9Pb1YqJWx8ZpzsfPp7Yi0E5hemMf0zjn09GcR79kDRMwzSUG03VJmwqBVWZzG/JE2wuoKFHIEw0iJTKAVcMwDSvOppdWlFZVLtSutefSvGEJxKIV8Xx7pfBbRHO9fwnSOSRqIJBSYEMRRW2hgenIetekayuWGetxBlfeS12IBlKNs3FynCRwqoPN/3IBMmy2F5J38/7P6bE0ZCGUDDKauweOWfV6eYr525ikrySKHJ9izshaNmXzYc+e9oa1KkIxi7aYSbvv+Zqw9p4ROcr+456daVoZL8HV27T+Ov/v2r9FodVHK9yCWzCPRuxpBth8R6pOls4hQNlifk9pqrsxkXe2YZsoKXWnFZ0X7Hz+UQIM67jdNtu1adlloub8tSH9TGA2NIma9MN0uQdTWC1SN4WoypsAk59uiMzqg0jn1Ak+dEl4ZQYigkzXh7zTCNuokm7ebGLzwbIze+GXsuu56pO/5HbKIo4Y2Yh3gueYUfls/jp1hFTc8cj8mJ7uoH+CiJwOqjXzBxL2Y8vLh+S99BqeeR+6sCOzJhNQdlEW0O0IUJZXqanuri63u0kkrzV87qWXYRITcyXiyhcAHL860U4VU0POMKC48ybSaayBTdD4UTkWRgC+dJFfHGVhCAIs6TbWlsUiJqUmPyaReI0EcKVJOM3GErS6CVUmc+fIVeOLmbSiN92KhXsb+LQcxPDIK5J7EYnlOWsFMfPK5rDYJwaN6dR7tSgUTe+LoyQ0hESfRnzO7fPYkgiRtskbsMT5jprRc9xyuoMMhrVhsjI/3Rsg50WvNvtaRHo6iry+P4dF+JEdz3McSGuc2iVLHmeJGHa6TuPrU88cWcfIwjb5NkysRMIvhZ66ArhEm4UJDL6bCMcQ6PHVN75ubnjRVM++y9cr/cdZXgoZKnwlW8tQzQUGfkUnFhYGCZQm1lN3maQYNnP+Gs/DzH9yP5WvaaOOkNg/XNv/LLEvYSLWKk9OL+OCXb0Y0bKGY60cYTSJfGkMrKCJSKCHd04c2a13SOpPmwct619x0A/XOI27dKlsjRTgw+1hPA1VZ6lFlY07ZLK1P7yzyGnOJNYvnzmo40X2JrNF2ekhNytMw728q6nok9RTwZULPnm3jidR8DTrz8QM02EboyWHNfd9GcLyCfW/5HNJBTJukFQnxeOUYtrSn8UR3AX/x0Q/gvR/7azx77wtIVFKYq82ikKd9hkVcooJ8L30212wn15csGm5Y3ghGVd83830/RTmv8+NaHYymBCwYjNQPTtKGkekigTDrQYvwH7OUlgHPExf483QmYG47MTGpxc9eMOs4WXW6WtvkbjquF26iawoiAv8MOCTvV7hAIq4WXZXDC+0Welf1Y9Ur+vHsXS8g1kgikgWG1w7hvv97BP3DGSy0NqO3VNQzpCwLhc15zby28sIcuvUqKrNNLB7LIZPqRyRISXybJ6icnzhS5wYA+JyqlbptaJU/VMCgxI+lpmq9OcDKwDtiGDzpjW5AlFQTWgku1FCDIaneqFT+ewd60bOsoPtLjCKR5eB+KCPz+myIykwV5dkqZidm0W0Q/DSZ1zgoHMishOyziAzCtZ516pLRRz9gBlujD+oEk3KFUU3ZA1I7jrPCGnInRx4IYyHWvXwEyVwCv7zxYYyuqiAar+nAUvD0znyO8joztYh3f+ZbiKX7rL4mFyKWQ7JnJbrJAuLZAiKZNBLpHCIJU9mQwoWE+LtC4Bk0/PS7AN6E9bo9wKqSgJnToXWvC/2mtDrWC3QZUmrtnVMCzR4GFxTvQAFLv6y/JFKDyDCWzrB48b1TkhL0ZwlVGxeYIA0F6ViTVlmUR9rYcNM/o7VuFfa/5qPItQKxk7qxCO6fexG7oxVsCWtYfebZ+Nev/TsGz16LrffsQWe6g1jKUGJDeS0rsGsw5zfOufaV+k0e1G1mX8uLtkeXP9eK8emw/7zkFfNFOdhuQe5Uz5GR3TjAHCs0CiPfn5tX4Iy8ZiuiKdoQvtExfSrD96BAnI3HiVi6BOiJI622Bnu7bTGomMqSUdWNtHHGprXIroxg29070C1nEUsZCj20oYSHf/Y0cv0ziGWO61kxmPb09iKbzmjRzM7OmIl1bRELs9PolNtYPFFEMtqLbpAAurzOtE5go23SGI6v46RiHFAiJ8S2pbFKIU+b42UdZ+uLt8aGyPVcQDqsDYiE7BU71h6d51lmtMIGFluLKPZmMDw2gFRfCsX+IlL5JHJFyr8YZhHpRNCqAfOTZSzMlrG4WAWn7VqLvG/UvzJ1RD6QWo3WKXQ/NOcLtdt4vXSld2L46VwG0STQP9aH1ecNqwW3/cnDmDo5gdzAIR1ZrMoFIjmwVevfWZ1UG8DXvns7Xji6oEDRDRNID64BkgVE4hlEklnJ10Sp501AjJkWNyuzJ1JGZcPqZsV5rQQAHWnII/PKfk9s+P1Q5G9q87imtk4hl+Kq1nNpkicJeLjeCn3H63UHsf7ON3cMXl9fGrvE+KMaIXQSI0JOUVedSznWWrOF9de8HvnPvxc7r/0ickendaM4QHXf9D4NGdzTnkY0XcQ3PvY1jJ03hjWXnoVaO4bdjxxApBJHrEVU2VQVuJGpjMHTdXhoSKemUn1GOIdYE5klt5arq1JbVBptTCjr9Zlqvnn8iEXlfl8b1IEjmgoSPbKNSr0mLi1V/0I29Li4iJYWcmhUjV/MhyCvXFdfM/DZAo8gQo2neErvX+8wXSaS3EKWCov0xmnX0bd2GGsuLCFsdfD4T/c4+46I5GKDWBK5lUls/uUWjK2bA2LzOvXUVuDMaqVGvwCEHTuhpLjI0qfeQKOyiJ/8cgv+ZNOfIuykEYTkc9sAQUvSvIZxcNNVax41tyF1lgE8pSnnw40u2mHcZkltOsurXri5Zke24L3RhtCpbkP6BNx860snE0dFHQrMcoRrqFybRyIXYmT1AMbWjaBvpBfJBIfFI8JiVK86HTLZhEgVzEAv9r0F+vAanK+xDioYxbbdaOD5hw8gbMZkU3L05GGkSy+awFMkoplkG4K3TIIBlfz4Q4eO4Hs334VnDtQZwsUviCRLyJQG0QwyOmkTGQ5+5MWkYk+XG5Y6VAK5JMrIAKmIgxgzFr4SueKntUeDF9ddGeYyabUdZGTlFiWPa388nw4w+UFsq+GMZaTC34EB4ipTv8lNZ3he8hIBwZ2EJlRudXEzbFgPNuyiGQ0RGy7i7Nv+Dfu+/n9I3/GkHlol0sEDs/txMt7Br7uzaIQB/v1jX0dvzxC6yS4GVpew4iXjiGRJK4sDrSjCJk8HXorxO1WzO41nMbJ8K2JphNF1FEXP7qJdZ5pm6gmcYZWSvJArO8m9eBdBllq1jaBMd/MG5mcW6djp2kldDUb3FovKNDrOJoW9Py4Cj4h2OObogBciz/Qt6ka6ohISACr055HuzyKVjyDIdNCttrBt8x5M7KtiqKdfgYenMp9LMhtDelkCd//sAZz9stC0puQcaCVEX28vjh4+gBgBNPka2wLn14kjB/GVb92iAY8zlq3HZedfiuH+lRrcCEO2sKz25yYNWKN1CM5YSs+U2tzzbCZW7cMo2WZ+3paoadK1x4zAYJ2KU3JBasdKrMCsX4mae0cIBVN3UAiLWQI5+WfTV2q362h36+hwTakHamm3viJsxcSRpH1KlHW4PSNtPjG5KDnEv0dRyPShHdBDKI1Sfxbl9hGE8UOmONKwA4G1NF//FJ7BPv4ifnTrA7h/60nbuNEUooksOpEU4mwPpfOIJXNANI0wFkUik9WwPliOsDxJmCg781kebrId4FbzksgOXwr2jb8mZORh9OBp5E9IRk6fTnLj+pTR+LvuPjjqmT74aRxlGfY6Rgk9hITeOoTWvE5PQdsCHtp127QUCIuFmE408erHbkJ11xFMfvBfEWu2cDLWxmOLRzCR6OD29oxO6He96R14xXmvRiKSQSxIKlK2Ig0E8QCZXFILvo0W4im7uUbnNObREmLOWiYamjGx5nEtbbHxPa/9w5TqlEoGvWH4JURaEzG8f2l0YvTR5YJzkx3qJSt51vuKJ+3IzUorHbXN0HzdeaGd5plGlhlXVhP1Kqd/aqhNLWBxsoGTB+YR6SaRjtLhjqbSRYFC2ggdo0SeaNBs+RDa4aJOr76eXm0C2Xa0OavcUrbACO8VGRKpFF7ctR1f/96v5AgnlROWPd0Qf/eZD2J2ahbxsB8B8ohHc4jHUgKXCPYws+CJKlAwZJukJblVugOIEqna0thewh0o5ytDcvOrEndX/GS3Gdg7d/RO8aQjhgxLTldahqwJiXSzlWQIPrEYvk6jabPOtAzxd1aWrG7diePsABdDn03RhFx29li7aKGnj1NfZFIxbW5henEPXagta5CAuRt6d84XGnSwxjJuu+cJ3HTvHgfwkdGXQDeSQDeaQoqbN0GQLiOnSyLNiVxRzz1wptogW44ySdpfUQ3fc237+WhlxIdWXxUKgiZClzAdYZ2gblLDn7AexJH+r++XuBpSJAueRg6V9pFRQIqTqVEqtiTqxdVgabbQSKncGfBSjbYwv3IAZ97wJQzGsnj+jR9HqtXGweos9qKMnYk6HqjNoBW20Zsfwpc/8LfIxPvRbXQQxqzWjCdipmFEBQ2nB9QmQZ99uyXhdvrmGhjEyOz1kj3t0IgWdhLwzzwBTe7HNHB5UhCgoP8rTzI1z9VfNAQwlkgtSalSgzmItJHJxhBJnZJtYaYh4I3AXtuE7DRZFdCexCRRO23LaAxEsTpI0rJqZ5mNZ4qqGZx06obIkPUTi+BE/UEgUlZfUPYligbmEGAC7yYxRBK7mFnsgycS2PnsNnzj+7+wWVG3mXLZND7/6b8wDnWtrs/FINBX6Ee7TiQ2jk4zC3SziEeLrn4n+GVtQipJiG0V5Wlrk00Bec8aZOHUi9W7PKlZtrCmlqE4gdEEHQrpR2TXw3tPwzdNn7khA6G8zpuIa4oTPv5w4X3jdVsZQvle8+ONJ4nSG1bBHrOCClNsAVdRAxejATKFJOa7m4GIlXnqtWbTSv1tHt0sWYzV1ZY964nFDj7wxesRTWTUOgqjaWWBNghFz6AC4pkehPEUYsksujECVQES6SwLGGV3IYOGRNJDeRglSP10bUNlity41uqhKJshhNLuWSS7x3pnVsSbgrpa356f6Taxd7iTlKk0h4xkoO+zfhEiSpZSzKlBOjE5L7XJfq5DqKvxDpqXno2+T1yLwtgwDvzBZ5CaqeBQewEHIzXcWz2KZ2ki1m2qyf937/scVvasAuIpuQcqlWIrIEqxO474uTYWWwhSUDDgbH6e+kskHKSM8K6Nau0MEUm0qU3DyPvWaqjemTl7gomxxY1q6cUD9G/OrZ3pFEESD2bF4m5mmUikhgusD9jsniLmE120wXFj5lg7xtBFD1Aw0MlqlKlVOqkNyZ+hoF09mEYjtUsqItq0Lr3nHDQXkhhITZqLdRFo8H3psMeTv30cP/zZwzrx/cZljfeRv3qLpchNow6yDUIsQwqP0k2i/lIMC3OLiHTSaNS4+eJIJ0tIxqkYGbfgGjJQMEAJ8zeBcmY8HGSQjxNJElaOkAyi1pSzDeH7MtUnF1rMKUer1byqgpzxvokb0ErVNpMJ2BsKTJDKSiRxoCUxy9vRQYp/56ZN2iy0PWumI3XMdx93oJGVh0K83bPjuuHPk7TBzUfLzocefwb/+qPfoRkhVZHrikMaZHExFYsDHOiPctMWkMwVIUVutk5V8yYcvZHkHQY1m7xiNsQ9qq4PD8MD46/TIL2QPjfGxmjDWoZEAd40W6RWH3qlC5EWPHFen8XYUUuULOcd4/Sil5QTtJmdsJw2uU5p46BqwDroIv6ZazD01jdKxXD6+tsxd9N9mOlWcaRTwewlq/D9Bx5U/s9ToTeSw3Xv/yKyhT6kYvbw+H0pChCdcywtcn6lcOhoY6rR2Cek4DVrFvXPDNP1LSwf4bSxGk1kc3kbR+w0zb2BKWCEFhxMobgZSOE0tQKbG7RJmWj8FDPNNqoRMrQAOKSeiCuFVbsmlUaHYmeOyCL+ruOu8nc1OkfyhZwBTAlSp7Bn/rRbqCdeRLxQA8u709li1BLmRXHThkw7WUe5z2ttszbu+tVvcMf9z4mkwV3Az7tixSjeee0b1DZJxpm+2eepafiE7x+XM4Iye55gDHydDmamZ6V8yB47NyxlhlpNysxkEA2LCNjUDSOIhkl02taPVXbTNuEBS51toF4sK2czyu9z2oqGb5wgUtargX/7GTHf3IwvFwNPcUmcUpeM7TeXjrOeFHU3ABKphDZHPJ0QOMn1zM9WDXejHhxUIObr83kR+SXzjVRbOtAvOvBTfOlYBB/7xGcx3RlGNdqLWCSp+6PWFdefDAWIHrP2TiCMJHTopLJ5taH47/9fW+8BZmlVZf3vG+vWrRw6QneTBQYVHRUJOuo3I8YZFUEx66goKDkjsYkCDTRIFgUEkSAqCGIYdRQwIIIISu5cXTndujl8z2/tc273//985YPdXXXr3vc97zk7rL322gwDS+nnlIsSKhGx3yMOoeh3ZPcPtGKfojFqIjTtxgeusFlT04LguRL57dqO4kYP5AAvtTg8TghIDTPSBymoi3ARYPTIDtJBwVpSyK81bPlvr7KRF161aqtmuf4he+HTJ1u5UbMtzYrlv/RWu+0nj9jf141Zg4OTSNs+O+1jX3r/J6yne9AbYJgTaoifR9DCrwFrjaaRqHGaTMCDzDjAJmTZrZnUG4MH5uDJqMlwRbV5B1WElAcBPH5WLkFIcLYXG0rN99JXinxpVz9wiw56CuPGmTDq9y370Gcvv7iaJOyhaFjZeC71YlZUGaUlfrPSSvVhdFgyW7J654uW6wYN9snyQmlbXG9d18uhFN0XD5xwMYHYW3vHrT+wJ558SYYvigS8ad/X2Pvfe4B6jCnfSRAAY5HBA3pzgZd4PNJSxMakwqJL2mgNYCwJ0S7q/rlu0H4R9MFWkgmbnJgUXpFJ9zGhzVL1y/y6HwAAIABJREFUTrN6v9YE701JLZPuslKZweCUtEgZyGNTojDiacm7iQoU/QlHcEWXUqmiFjkw4FoNdpLz7om4cE3ZbEJiABrfyhC9dCepprVyz1ijWVSFgByYlBCvifH0PNsrEDJ8taaNT8zYcSeebOmOfivl97FmGvZTlzSaLQmZBcOPYcrK8xLxNJkhjfgx15/rsFy+X/zubDavWdHqFmVSvUYf+H+JDasObkUScyXMXIkhL6CV2FDBI0YChbsL/3ISfkr0NuUxyoucNyqGh6Q6PTSGu+FRG8OeXAmwrWEsQY2mpT+wvy0657P2l7cdaZkdBm3VDafZ4x/5mnWUKjbS0bTmx/axzlyPffP6222qxJhtl4x5/35vs4P23d/6csstkcxLJZ7jK/qbRN0CgyvkuKJ9qvGBHMebsrlf5TzhcHGt3AeHFMMFwUI5OShqmO7HnNoIuPB9Ne8HNQiXbM1aMsiPKD8C/NAEc0Jy583y+xpwFQAsKSHEBmtNf4jAjfNjVW/X2ru6RI5wLJG0SmvW8ssnrZ4oW7az03JJJ+YrjggjWAmXNWmC6QREDu2pp8z6Kdn13/q2vfTqhDY4HVx8ffKwD9juuy4R8KYG+UxabKRCaOogQvN72jbHKUZTrF+sKDh32HnpGuoVBPoQiuf9eN8yRAmVV7ps6+iYLVm0g6YRZixv1WpDOTSH1yxjzToN9DQ05ARMcV+kN/CfAXZoXRTIKu1jmH6UCEO0E5r6FWJrzErWevsGLJFCsYW8c8ES+VetXJ2wzs4eJ8dkMzq8rXRWDRuUGDu7GRA+oAFt1VLdjjvhRJuaXWAcgaV6d7VCcrElWlnhR0KXpS4CoEk3G4AUDQ3h8JIDE3FIi5zSXpdl8p3WkevU/bglotRllti86/taUR6k3fcY8gANuQ6eJ+Y7ejSxKyjU5QTgBEE15/N6o7MeHlY9jF5EfS+WUvBwEgoK7CbqWQtLu23lPRfYlnt+YYVLvi9v0H3fBbb1+4/Y1I8esblF3db48GtULx0vVOzKm+9WEg903pdJ2wfecZAI7r3di9TMvFBJ2pLh5daX77bezn4RCogGsGztHAkgJBIHQqnB64aAQR42x3owhwSkNBDUnEIXROB8spzrbkUxNRk9dSo54uvyr2EMpNDnbfNxMWSy3FJGCLNz9L2QB+sgU7pxZJBpBXwWXoxQvNwat6W7t0RwTyMrCkDHbCQJAzipXymPAMG6NWsVhbEwmmRLBTA27ao119q6DUi9Wps/fvYZx1omSU6cFmod66tKRwJSLCMdpFecNBLeNxArFH1BtkFzStMJ3BjyOjWuBG0yRWgQIrX2TStXSpYipUh3WXdvh02MT1mxVFDDAqEu6U5P92Kq0daRzlujlrZmnTIVOXbKki244DCmcqEkaNZqJK1Uqemw8nwi4T+XT6nubNkZa6TGLJllVnLShocHbW521lMjvDaeMzDdxMuGmVUq2ab1I3be6gvlQYnkrrxmrX3jkttsrJjzHBcvrlZqB7UQKEDhJEFKB91L3VLqnpfHTeIMldfCwmKfIn2TEVKf2LDy3Tq4nps55ByZIO4cnT0lVYmga8ufPDCmA0TPKog+kCviQ3PAJgh3ydM5isyXI4d1a0EYqDatvHjYdvjZ+bbwlxdt9PMXWa1W8gHXHz/ABj/+YXvmE0dbaZ9lVn3rjtaRzgps+P0fn7Cf/vbvEkFLJ1J26H8ebDsOdlulVrHRqSn7ya+fCMqLQqiUO+XSHfaFD/67dXUusVymV/cFcum9sRwkV6NQqCpUzw2Qiv/UJhM+psS5o4B+7oFwTmxqDoka3mWQ3EJXar6JfVZRUSQIb3DwvAljIFG2MFA7lekUKOb5l/NiNa6TcIuylXJgKBQVG5sesVvvW2uXrDlLlEHCdcA3RRNBJsbfO+TNQmKhpTI/CO/mHl9pS6Nql152nY1PzIu8oKjIzL76pcNt0ZI+AS3VMmNMaPwvWk9Pv0Jf1irqZeu9Ei40KNlWoopAOIH0QH4psC/pAgc+LdGnUYisH0j0GPt8vlOMNxmFMP2PAxJbM2nw6EOZpMUYWGRo8cQcCed7K3SnqQMZWqYaVOr20AO/s6mpiu20bDdbvnilZTJdajKYmhux10JvzBeF1itqKpdCAwkH0eVk4bk3NMKlYV3qKOMMEIWZrV59qW0am1KE9G/veJt94pOHCYD7yhm3WLHZa0lEBQC1WhlLZ7g+b5CnPV4TDpizVKPu7g39hEmIxXFWUmlem2yPn01sXHVwK7a/uXV2TxDDYB3S0J4WgSQXqHY1x1gmwkT7wXfBK6G57nv0ED3E9AXhSwghsXu5bvbZf7eBr33YRn/6Oyt84zuWalat1KhaK52x6V0HbOdrzrKnDznW0oe90cqD3knhIFHTrrzxThtfQFKlZZ2plh313x+3cmneRka22s8f+7vVSGCouQUADkNy9Gc+ZP0D/SpBqLUrge4zfOOSUNcowQqIA7qraXoJDh3IZNpaVY/5+X42xxBqJ65kssiXcvhZP8JuR4Ep6WgtABViCCxEPkjdaJVcA8tbCYPUjvS4XNpFggPNhm3ZvMme/efzVmnVbLbARPWmGFYnnXGMLVm21IaGBnWdAvqkEBEGlyn4cjCwUa/I4HCASWXaoEerYasvuMLGJuYUVcgAJxK25pJvmCUrVipWrFIuquXP1RvrXquVfKQ/b0UW8V5DtSK+fyy7qQElGEepVgRsRfcYSl/CAEI0wH2o9Bb0uXU4SUPCVADQZxEUQq0YOVRE40HUWXOEzhFWoL570YVX2eZN04YIP4CVcI1Wy978pjfaRw55V1t0XDKv9arQZxBjUiL0onxNMCTegJJN422rNjszZxdfdoPqtRiQq9eusc7OjD366ON2y3e+bTa4r5XTSy2R7LSmDqU3FERD53xlBUHWEM8Aznc4i4jo06sF15oDzjVv3uk9LZgtCmEDDUBaSm01gqDIGObCbl/XBVSIobSTWNw7RQ6o8rSgNuBaVds2CWB183W72ZKLv2z1xXlbf8r11nr4cWuiHs7JBNxKJm2yp2W73LPGfn/lWut+80orUzMLnkSDnusNu3jtbVZRIGe21y7L7D/etp+V5mbs4f/9q03ME9pGzVqTNTv9a5+1VtMbDBQ5AAjkctJIjhxnvBQHUOUX1au91KB8jUhB+TxgCG16jvyyMVmfSLrHKLCJhJsjiwrpQU7ca9gCIeH/8vfQOkk47fvVDzC9uL5RWlarLNjzL75sv/7V0wq5sEllapbNlh1x5BH2uje8wRotn0b3///yFkG8d0rv44d32yRB1iGZaNk3zrrYpmeckM+9otB54XnHqwcVcKi/t8d7mBvetxrr/qrZB5X+uCElBk/Yx9wjPLV4uH5YolfTBIJQEhPfuwpiT4Tns4UiCBijvIijRDIHNWzX8Mqonu31bmicTsaQvG8I4zHMZ5xxkVUqAFYJNcNw+EGM/+tD77bXv34n6+vp13NCk8taSOs6FRUGkz6bZ0GRJtT3wQF434VCyZ57caM9/ue/2gc/+J/2tgPeaplswi688Ju2dWSzdaQ6rdq1yuazK6ya7vNGnGDoVM1JYLS9RIaFVfOKhOadtAPSzIZRmEz0tGW397dU2lGZxEO6qObHxtIhbHioHBdN7p3NEaQ6faO41i7lH9BILaAGbLUsn0haIVUXwpy1rI0N523n606x1I6DNvO3F+wfXzrfBsoJ6yDcTDlaizebt7LNZLO26q4z7YU//84qNc93/OFnFK7NzEzYP9aN2b0P/14PIJNs2pGfOcxymbr99ann7HdPQ1NzwEglK0valz9zqK1aOqAGb5DcwcEh3Tebzw9MnLVLmQrShiPpURfa4xsvX4kwobEbnrtiqWmfYwOCYMuC8qlhc8awLzZpyHNrTKWLmwnND03aMUWJ10bP6sYN6+znD/9eD1Oc2kbLyvWavf9D/2n/9q53tsPKWBVo52J054SculGc87qr5uY4SAcVMZlu2WmnXGAzHNwUYFXN9nnta+zzn/1ooDnWhAADRnHQi0VvZ9REwoWFNuIdUXBeV6b3NsizAA5JjzuE5tG4xDq5YyUOXqkc1nA5XJEnQsqFkwF0WrR4kXdKpTM2NzdrOcpDon0CInUoraEWy570mnenAKTTTrkwpC2OHWBkcQDHn3iEDQzkBGIymRGVDQxbjJTm52a0p1XHD/wDFxwEXUcDu2StTIdSld1228tq9YqcwAknnGLJRsu6u1E3SdlcJWkL2QFrDPyLNRLeiy0pJbfVIqwANMpwJiCw8HlEE+TB7ky0h0Zf85/AAG04P6KlEagSmpbyZBzrIxJGQD2jNZP8SMo3Pkajo9qyUqppKRQsyM2olQ50Wd+h/8c6Pv52a+Sy1nh+nf35xDXWu2HaOgiRMklJ1TToP1T9sGXVZMPG/nWJ1d/zWsnAuEay1495oFwrG4b2tkd++yd74rn1eigrhnvs0P/8d2tWq/ade/9HCvCx3xVA4F0HvtH23nUHW7FyRXuwFpZfPbsingfeqiyrh/o+jdDXKW5MdVKJk+tKDIpZAlPLJ+wBvhASbScuH9IQFp+NHME68jDE5eSJ4yC1MHlBZQc1MSRt8+aN9qN7HxaAwUEEZClWy/aGN7/JPvOFz7cxBO2D0Jboid82AKgyP2OVYqFN4eW6kbKZm5+y1eeusVIZTB5/nrKDDnqzvffgg5yjWy5Zd75L9++dVC0bGxsTe4swlwNIIwYGNWppd1ALRe0j2+GkmJD/ekNBRgeK94pfhPBKDXgeQWhBIX/CVEJiMBpjVYRIB9aXk/Pxslmxqij7eT856VTDyRnNhgQWzjvnCgdnE16S8464uq0+/1SrVGbV0IEoHNMPCaHFvZc6p0eXfG7/4IDNzxeUg09Nzcgrwo5Dfobcvb9vUPf76KOP2YMPPiIwFRwFeqeUK5Mm9tTXTz3Nnnl+zH7+u2etmuxRyZP7zFLfFo+acBlHiJF2aqpKhOyxrXt8UG42InyxHuetWWF2DhBjyMFizushoqOf8soa7NywCt4tlbfGULelX7eTdb/3QOveb2+rZxNWL8zbyJ+ets1X32d9r45Zg+6UVMsytTDs2qOENkd6pitplSMOtHKiYnXxNgHQOLx+XRC6YymHDpNLrvq2lZuEl2Zf/eInLNtYsO/e80uroiKhPl0ecMpWLem1zx7+YXV0KB8MaLKoiiGP8dw9KCuQW4mM79ROHz/p+Q7ibz7Eyr0qG9jZWA68ONjgTQmx3hdTCT+4/uVGMciqBE8QsYE445Ue2OnpMbvz9nusWfPaYZl5Qo2aLVu1wo478QTPo8OwMJDbOJ+Jkgj1ZeiD9QpNEOTyPlyK1/f09Nr4xIgf3FLTWkmogg372Mc+bG964x5+YDS20g/cyMiILVmyqL1+3HdsPyMHjjREMmuRIljj4DW3XwcOffTWREDkjJHKiPeNzkFSMmGWkFjeQWxO5TFAPRUBhNK01TKIIiCqCJgSaSNvxxx9ZqjJO0OKEg+G+vQzjrUEWEeSCAK1EPSrnRG3bcZuRc+X+49RhI82wYgmbL4wKwB02bKVVpgv2SWXfFPItvSypOjZtIVGRVHCRz7yETvgwP2UBnEQy7Wm/fXFMXv06Y326pY5a7Xy8rKNZMPBMHXree1ZSP6WPT6g+6UpQPUkTS5rqd0IF69NhwIFAARehTfBK6FG0D9opXzScsO9lt53b0vvu7P1vWE3a0JHROkBAGTrlI3+5Vl74eYf2cCWCUvXmpbBgoiUHtkgnuxHaZLYjTT5nl1t+rWDCr9J2Fl8wrLYi6m+23TW5/dIkydpN996p+2//wG2bLjPuvId9sivfmMvbZxTWx4sp0SyaR2plJ175jHKVfEO1PrQMJYqY8aBoFhjxkPIy6sjxkGVTJDWRLMpJ3kWz1lbLZeEAQkFuo/AHd7AvbUr9XMgvfHCQzXPD32wlw4j9cFORxwhDhB68/1KdcFSiQ77/f8+Zk8/8fcAfDWsSG0y32GXXHZpmDcTR4iGubNBwRLomzzXieh1q5aKYqoRTUDIGBndYFeuudWKiLgHIbavHvkZ6+/zaQYeaTCipNump6Y0FnN8fMyFC8JYFU+pXF1C9yvlCTfGiA9EA+b32Gld+bzNzsy6sEGpqCYPfhaNIx5GgntCrr27yc27A1QKH5NoeJUsq95hNrP/DmGlS/Y2rb9/wDZvHbXV513Vlqd1XnvWVq1Ybp/93OHaG5AcYrmLkBnecFWySt5LrnUI/bdxSh+lrpjrM2iMa5iZXrDrvnWzJZNZGUX6zXlNVbX3nJ122slq+O/tdVGFqenxtjh6odK0YqVp9/3qeXt+S9GmFlrWQjkDZU6xv+qWGNnjgy1CMMJJVIYWmg1LQ+1LmJV6MpZfscRSb9jd8rvvaLmVSyw52G/Jzow1QOUysEV8kjj/y82WbeOTz9qGX/zWEk9vsNx0yTLFqjXSZpk6OXQ9dAGR7AddWno7s3SZBMoknpuSSm/Wip95k82kK9JdwjPyoFm8uQLMGTaBWXffgA6Kt5Wh0le0cpWQrttKxYL9+S9/sz8/s6mtbkC4lkulbPU5xznNkFJFBklOZzl10zNbZtSHz3SN+SchICEX5Q/Kz4R3YgIVGG7sWldcKCwf6S2HDhYMDRzwKFmjRosgi+LSrp6zcCgoNThzykN195z00GZF0MhSOrOUbR0Zsx/cfo8sOb9XrbZsslywK69eK/pjDOXFtQ3IcIUh0uWSIgcpKyh3Z/zGgkLCeq1iU9NjdsXl31EDg2eZSTv55CMtnXZ1TAAfNQJIZM37ZQuFBa3bkkWLdI08lwLicFLmN+Xh8sahCYBDENVBkEzlIGfDNEKEyksLBT1jhrSNEoYDOIn5tU0TTOURFDxqNevt65PHJiVD4havqq7aIDKPfI5SmUbTXl6/3m6+8S4dZmq3KgV2dNiH/+sDtudeu8i4w8FWGsOYmS5C4cmQLjniLYMRokz2zczsjOfBoU2UfURU9sjDv7G/Pvl3HUxNWgy6VGTNr33d3nbwe95l9TrGpsN2WL7cJiemvZEeIK9WtGwiq8aCucKs1ROdNjLWtJ//+Vl7ZbRu89Zjicm7H2hl+rots+OwZXbocxK0OvcJo5qWZLQDOlOlqhUnZqw4PmGFZ1+16rqtNr9ui1Vf2GT5essyADpYA3GAE+qrTVVduUI8ZCB1SbHAYnIKV8yXQQHdUnqiPtOTsspn32YLncyLQYXR66hsHhXwo8wLaHjKNWdzHZ3KK5B5RWVidOuIVYolW795iz34iydDkd+nHCQaLfvmxWfoUPK7CwvzwSPkdIidoOJhr8TQOVzBa3Ko0VjicIjHvb3MrIZGeV0T1DSyn7hXCbABPqElHco11DhjmByBKZHVU7mgtJgXM4rrUSN6kvpx1qbGp+zG625p85OrlYZNFgt23U3Xa21iGCe5sEACATBsVEGSg/QJoTlaX+UFKxYWlMNNz4zZVVfe5m12ut+UnXHmcd4QENacziLWgC8iFbwjBg0pHQ4sX52dNEl4VEHLJlEN3pZD4ioZfvDcM7fkwbhvgUWZtA42/8ZYi0KriY7uob1P12ca43HRv8bgOSHfQVS6wHg23jCDyob3mj/x1JN2//2/CGqWPpWQ8P70U08ytlK9XtHBJWTnQzNpIqKsTU5NKoUSSxA0GK/ZRe5e9AaRQOGN0xtY/8suuVa8AOZE8QBJigTCZdJ23PFfs3QGz+nenCiCz5EKB6owRHFBuB5RORDnUrloOaLBWkrhf2Ju3dOtRKFszfmyFbaO2PzzG2z2n+utsnGTNcamLQ90XvN2JuW8tGSFso/mnQSqIIOs1QGDtwn0t9gGFSelCUmNyhPqg3RVBcKiTpC1tNnL6ZrdWt9k//3lj1oyBz+1oBwml3cAJDJusGoKM7p7dCDiYGEeNCijxHGaTXv2uX/YAw//2SoisGdU68tlknbc146wFSuWtjVx2QnaJELWyUfTVizhdX0mTSQ16MDCOop6VMGbxFolHgwAAtlOVSbaA5uh3/nnx+kKeE8JxakU41PpIRiwebhXjd4gfWm1rI+pgPB+az6i8/qrr7VEM2nZdE6o6VRx3q656QZvRQylJZL9tnEMqDYHq1YpSeGhiQepl2xiYtx6u/M2OrbVrrry1qDVxBpk7JjjviSkXrV9zQRyCiiHj9p2rL2io8XGXLJkiU1MTbjxDqJt5K2E0vLAGimSF/WP+wYU09CtZErfx3vG0lKt7lMN+Wx6a9nc1Mw70WzSHF6vZPjfnf/b3d3lhieTViSmAW8yFFn74X0/tl//+n8dmMphBLxF89zVJ2ssCXk841kgzfC7maR3xnnpzjW2eXZ9vd02NTWlZ0sEpucnkgwRUNNefHGD3X3Xj+VICO9pKPAGiabtuc9u9vGPHyrwy1NPP08Ab3FWcmSjOcbhyqS+5kgCe5SSeG6PtwsKVfse6ozUEUVXdM8oUCGIyIlYEb6ilKWHZZENtY18gcV2fSHPdfiSWnxoKxOoxWGSQkHT5rIp+21y2h7LVNV1ctzXP23lwoxyP5DCyelpdYSwwdkkbHDQxu31o8i5uCnQTz5306ZNCqXuue9X9uK6rQpRIXV3pBP2mcMPsX/919fJikt8K1Abe7p7tOHkeekU1fDk7YTBlB46M0oWMqhO8Dr/ooxCCcOHNbdVNxDOzuVUQBe3JzBj4uKomSMYxO4er5UK4Q80SgwDh1bheXHB7rj1eza6ecxy2bzyp9ly0a6++QYrl/zBik4phNytOmR4WX7CZO6rUra56Rkb6u+2mekJEU82btxs1157m8+HSpjE3b961OfE12G9o4ER2URytH6v8kKI/pUrAvyQ5CFHdxpnwuhKwqty3RxSIeSphO200yob2bpVLLA4VMw1rb03Soqhkjjy0ZzbaKo+xlPU1bBm8IsLCz5cnIHogHA77rijQl0OELjNjTfcbM8++091FZGeYYzz+R47+9wT5Ol0LyIh4bmzNjc14cZCpT0veymCiXTe0LvuP3fmE3nyfff81Na9ujk0X8AdcGNKmnH8ScdIXkh2MJwnnlds1pCoXWjMiHs7dq1JXIEvDu7fd3l7S1aFsC/U9IDO1U8r+UpnSMnbhhm4PhOU/CUucuhOidKRQdlBnxFqwRqiFUTW+D7vV0iYbUxV7c82axtyLWuB8taqNl8u25v22MkOfPt+uiHCRQgQ3CAT75jAjuedmpy0TsoMCcJaNk2XvFFvLzKkjNPskKLjn578h11z/d0CJeh3xOO+86C32CGH/Jdeo4bqQCBwEAjrTtO3o67Sygo1bl8PBxpUXwxsp8ikicin5sCGecB8hq83qDRtW2HMYmjUj6FtDGtl4cXEIkzyMN1HZjiSzAb+1c9+YX/+wxPSLyY8nq+V7AtfPcL23nufYFSo/XmPq64tWHYRSAANaxWrV2rWrKF1PKcG/C1bR+3SS66VvCpe/i1v2c8Ofu/bVbNeWCjKiGZTaZuemRGxnnv0JndXT6SWyWu6uvOKFiIqTq6D2J4a+ANnm9fxO/wuh0jN6LxPB7N4UbtwkbyYctAJDnjFmvhasx5+cJU/57tEOxSpRs7AmzHUxighw7RdftkVMk6u1AEWkbRlS3ewI7/+Oe0Xyb2GUidhf7JJia7Te8nTSf3J/YpNTg7c0+1lsXAu8p3dViov2FVrblTLIt6fL5whTm+XXXaxQw77EPRkPQNO1PaOh3uSgQ57UVUGxoeKiaeub/f+mOAnV+wvBQyNDNmuTqlDGw5mRNO0ELh39ROzeg7wYVFSWB+K62yMhtecKImQm/Lgs8m0zTYqVutIWWrVYivsucieWZixB37/uKwPYIFarMIcWcCco796uA4PIbl3eqRs6bJlsv6O/BGqzCssZTMPLxpqgyIgeXScIEX6ysYNdu7qa62JymDSB2qtXLXcTj7xCOtI5iybY+yDK1q4z0zooWB1NOM1rIUsv8Izn1zo9V1XamANfZN5eAXgw0NwZNkR8RgWubfmMHmOGz1tO3pRLdhJJuoECaqP4q4GttfLL71sd91xr6WYUl5vWalet30POtA+efgn2yUUNTyEkp6Xspz9QxkOnrLVncIIQLJ164jNTM/bNWtv8vJW0+wrR33ZBob6LUekEuIJs5r6pNUvqwPheeXM7JyQ20gsiQO4AXySrIU2IdEAtVWXtVUzvlKUvA5ftiNjC0Fz2mv52wZno52t5pagEaWy5XaypdK7Ar+AaqoSl6tYoMpJOMuzuvTSK2xkZNQVP+T10/aW/d5oH/3oh937yXt75KNUp4bCSF4RF3I/7DkcCRRNwtply5bbxo2uQ6W5SY2Kbdo4bnffdb91dOa1z7jGBdDyjk779KcOs/7hPpdI6uiwhdkZvYb1Y9+7MD8sDJ/J7KIPoSQLkh0ObfvgeumD2l0gGQQ5mfbBDQQAWQNCXWlMIS3kaLQCZaRbRHxvWj3RsGZ3hw5poydrXTsu1t+ruy62Yp4e06QtTM9ZpVy323/8U1kVeMOIVZMPiNFUqdgXP3+IDfR2WblGWJyQFacPE4V58kg2zfTMhKw23+/M5W10dLQ9e2bz5k120IFvs5nCjJ1x5hqbmCyo3MB9dHXn7MLVp1pvvkfavpoWD8ocvK3fO0iqN1XH/IwHyn+RqhgPrkJdqX94Ez3kBCeLeHPCtoPrDClZ0TAwTQIFgeIWYiEPP4M4t09m93wsHtz5uQW77JI1AlDUcNBoWe+yxXbGmWfrWtVmp3JJLEU5G00IbzphCzNTVizMyIsNDw9pzX7/u8ftlpvv1OGrNZt27upzLNvhhzaWSBhDRxrQle+yufnZdhrEYY8jVLlGNjyhJZUEvDkGItFsiNwwPT2jZ0Zk5GQJb6cEwALRlv5ZKMl5bTuMlgxhMT+L6UA0hrl8t68nayREPtS5ywBOXgM+66zzbG6WecKu48R6nHTy8bbNwWmqAAAgAElEQVTHbjvb2PiYT2+kbioEuGEtkPhwPaXinMpy3NPs9JRyV6538+bNiuqUE2dS9u2bb7NyyaRdRaQoDKBRs4HBAfvCFz6pzq/ubk+FIndcVYWg8SZCShFcB/qnt4xGFpw0wMKA7sSTK/d35hT/C7pRgme2G5YVaV78EuPsherKEzSsmEtasi9vM4MZm+1MWKMvZ4munKV7UCQEmnc3T7jXSieso5W0JkwUelvmS/abR/9s6zZPhPpgr1WqrrqByv5++/2LHfDmfUUOTwf4HlTW5VOj+FjgkKYResuKuQNwwGKA6BFi1Vslu/CSG+yFFzaKLcRCQB6/5MLTESG0RDpq/3rYFVMBGRKQbMm8OpLpBBXnJgtICdPzZP2V6/ng6HSH82SVF0ZBdhD3KNcjHV5y3RD+BtJ6BCZ8j9Jp40oeYglJRdEbJiDqX/7NK9XBIpwgkTJY2ZddtbZdP465UvTokigNk80b1bL0lCdGt9pAf78Oyy9+8Su7796HZEQofFxw4WobHO63uXkH3Pj9DjWsu+ffOjqqTQuvl3VgPRjclksnbX7ePTAhfnFuzhqAKxna4jyEZeojXkXjV6gpKyUCw/DSGOuIlxUoKgka9lAct+kgl7P5/J6kl0bomWH2jk9713NGUUTPqmDnnH2+Vcre9+yAUtouu/xiGRfRDquw8ZjMkFMoXFVJ0D17MuGcZb4Qkfd+aq+5x9IXf7/xhu9IUL6js1v7gSiO/fXJT33ChgZICXx+kaobNKyEFEZaz6HfV6qkgVYcS4UukO8OUljNn1btTzFGVrWaBJpPqkgvACKMOaynTPKoGbxfZ8LSOw5bZcWAVXqYMNC0Enlp0JnFIuFBgemxQjQnk89I+yfwnRU+ohvVqNvk5JT95IHfWJ2ByTnGUThyCsCUyrTsy/99uAAgWtpU9gHgSbvYF1azo8NHHPKzwWFU+BMmnWg2BS1lTXpgG/bkX5+ya2+8y8OrdEpDmc5ffaZlMjWf7RsOXDLrVEIeOkwlQvToIWUs2sOsIdlT6vASyPZfHiIH30mdMhA2hH6HAeGANF0AY9IiJszzsJqNKHazcno2Laiq52SIrZFSeD9x07598y326qsbVQeVbEAyYZdec3V7M/D4I5LP1cQcmmiJjQzIt3nDK1ZamNdY0J8++HP76UO/0rNHB+rKtWsFVM7Ozckjo1jB78SRK+R3ceNFD0hqUi/7QVe/q5kMqBpCirOiHgqdpuUTAQMqDYp2+Dc9q573aW5wkGfNh1nBUs9QJxGlFUgyPgiN92Y/aDhYGPzm+sxuhAnrp6dn7dxzz3ckmoMIut+RtYsuOl9MOxpNpECCXnMBbe2MJH6IxNi/1JcVNaEXXXO6LV/sryg88be//dN+8chvJHkjrx+ihaHBXvvoYR+wTqIXqZsglMeM3EhqaVl3l3tz4R3pjMJm1fzDJM34HCNnPvHHnd7cwtPy0DPNhC1Y3aqZhFUHOq1/r50ttWzQios6bKZZM+vqsJRKCPhLn/ZO6xGAUnFmTjfCDBUAGG6SBwBXlUXhQuK0MR2erIeCExMT9rv/fcKm50loIIZ3akwI1rhaL9tZZxxv1qhYoeggCP8pf8h3yqry/s4VLdvKVTvpYKmpXZPbQCPr0oJCauTo486S5ebmUfM/7ZTjbcnifpVFWEwsp5DYdNqe/+fztu8b/lVhqELHunNWI7I+PTOt2T+AYpE2mZVkTigBCb111g6GUGUwjXRxcEHzlkLfJz+LpAQeFrVr79bi4MY8mfAOPSQUIFnPhP3pj3+xe+75odg+tIpRq117443tvBlvHRk98br0WVnXqtq8ZbO8R193p8Cq226/yx7/w5P6/XRnxk465RRFMOwN6qHkwXEEJmvERoNGOTMza3vusYfPBgboq1VEzKDEQTPDYL+TZGCW8ewJOVkqjBesN6K7GBoDAsE+Ep4SZtDyORFoEodZHGSK+97dJcE5rpnwVwbXx5FieNl35KCFhaKdfsZZDsIS6WQyttPOq+yYY76mKIz8ER0pDNj4OBEg+6aivcs9VUpFb2EEoKOVr1jUGm4fyn/rmpusXKyLp43KhWZEJZP20UM+YCtXLRWSrxwWOR3uLxBvyHdhyEUBOtdjdsCP/aIDLCDO8ReF0D//xCEtDqmhDtiXs3R3p7WyKUH7XT3dWox0i1EIiGjCrmqoN1HaRaG/dH52ToyoqExIo7dCmHTa8l3dbe+NvjEbnwslb9V8n0TCRrZM2e9+/5RALjGOArm8VK7Y2w58k711v9fpYLF5RLKoVq2/H7JI2nKdPfJaGJHFixZ7eNZqKnf76xN/sl123lldSRzcY084x8pIodJHm8nY+973H/aB9x3c9m4sipBO6o5SE3QtJaGjgafsltZDajYbQnGxtxS0efsDIotMbTvwmmWwwgQ1IdUB3o80Ov1uQPCrNe+KifmNpD3xEhm0f/PWnc/bhvWbhZSqFlqpaDzIFdddGxQPGS7shiSGlfF6+O7gwKA8VKVcsPmZadu4Yb3dccf3VYME61i0dLGdedaZAlbmCgVDXoaNxf3iDWP0gAfmGivhcPmwNUf0ObxEFYipwWQDvOEZahpElDYys6WLh0SiIMWhTMSG17jJYPw9WnMRPkJuIiRI/YpaNMDc95rTTltieLH5yUHZXzxH+mVPPe0M77flNR05e8c7/s0+8MH3e5seTQjzc0oFXC8Mj1uRMdLhpSxYKstg4JW5Z54/pSUiBwz5zTd9zzoynS5HKxS8rNz2S1883OqNsgw468PaCMRUq6x7Zp4vh5k1rtBRFSYVOlaRUmqnUme4hsTdV50gVDnmWq6P7GR6nwgeWDRhrqjC0DBqMlLAiO2xevwZ65E6BNKHNRsaGvJJbqGJXu6e0LzKFPaWHvAjj/zOKlXCVAJF16SqVetCHo86+tPWCrNyya+XLFtm1RrT2wGuvM7a09trvb0Dbs3xbI2GPfDAA/aOtx1oiRY6S027/Kqr7U9/edYyGebpJuwtb36TffmI/3a1ytD8r4I5qJ7a9OLwMsZpOgMGSwuQoCl1msCHd2H+q5MouG4HojwfkuVvxfIPyGWwoGrf2zbdnVBRHTTybhkh4gJhNNoyFMI1tCorgkAuD/GkaeecdV7IP/01qy+71PqHBkNrpQOlMe/2afF1MaW4xl133VVtkYBGk6Njdvmaq2z9xhFFJa/Za0/74hFf8p7QdFoHi+aBXKeP3fBD5uioDkJob4zElMgG0kFGqI/QmQYOt2xG+BtLTGAlDgjVrYqGV5D4ZSN3d3XJ6GYyQe5Xapo+j2lsfNzXDGYZ1Cf1EGMQzdcII0FzQb5bA9fOOWe1vJy8cCppRx51pDrEmF5I9MM1k8viff05IgnQtMIsA+U6bWZmRocMCdresM+Q16GL6re/edQe/+MTCnmlJ8UggEbNPv3pw2zvvXe16WmQeL4f21aJHreN/4yht3L60EEmkC6kEBhOTZlkgDhVi/uuObkVw1qFs6F1T4AMlEAU9rarAUoJPygS8HssUHTnvG5qckoW0KmECzYwNKRifDzQcVwjUphefmlpmNWr6zbbU0+jLuiWqMyhltSF2XEnfjGoaTi6uXjJUt00KoPk1gIzmi3r6xvUweUQR34s+QjhWrVcst/+/jH7zq3f10hHCuWrVq2y8847r93gz/06Z5q65YKsMNQ28qVysabQT8oP9Zo2sTYh4Av86HLRXnrhBVuxYoUsJyGfT1v3QrsAIrE6nSmjNY1lJrxPoiUghTxLXGV5fS/bOLnDSzTpVDYwqqB55u3Ms86xwpzLw/J12nnn2bIdd0Beyz9bAE4YKRkIIXgtrpEQdGCwVyDMb375P/bjHz9gY5N0ppj9x3vebfsfdID1glXMzwvlx7suX77UXn31lYAB4G3CoLVQ22ctZLBoZaPHN5SveM+a6Kt1l5RVe1/Nli6lvFfQurPmZSbC5xgxilF34CmrAV0enemrCXhZsE7V2hvyiqD/aooP9whyK+yDWbSJpD366B/s7nt+qGgBh0LIf+FFF3o6orDa07CFwoznrgCkC3xG1hbmZ6xRcafE/TJOBoWVQamNgOmYXXftjUL2yaupS6tslO2wo4/9iiRtOSORLgu7bHx8XPtGHPcAlnluD+rskR4YgqRZG6RSOT0v31tpS/zoutP0xHWKQ7VOmyBMPI8oq48/SFilVG43F7NIGkhNrYr2JkTWVOf0dii+D9sp6i3zQDSqEgHrvC+oUFRr2dxC1X7y40esWk04Yi3yPCFVy17/hl3tfe87WA9d6KqEV6HI9Vg6l9UNUg4CyYtJPIsDQV2zS8slhV8s1rHHneyT0TNJhTHXXHOdX0NonueAsHj851I7XjZotpLKQ0UwVygPcJBRzy8US01xD/kQy6cWuJCLcX/R+6YgNwSryibyzQkguC3MjkCPb0Lvc63VaMfjetzjduTz4rR+85uX2+io0+94/eeOOMLecsD+Mn7xMPtu3/ZvnmE8uJVq0cZHtqgDa82Va21yqiCvdPSxR1tPX6/kQjl8REwYLs05azo7jY3mU/x8OgCRi9ZfIuRueGK4qrpk3YXLBZIlUzrAgGQ8b9YYY4j353mR/ij6C/OdQKNBnXm9lESCogp1eQ4uho9n7FGiYyUut+vo8f0//In94pe/DtMinGNww403WKm4IGE9ACmuNYoDaO01+QJJ26rVSs5LJoxm5pK8ovp6MTglu/ZbN1pWoXnQA6vV7BOfPFy5LXVfnS9IS7wnTADx1h3gigYpEjA8vHf6J9zmeLAdJA2i6D/81knbBNFbXjNTzlKtiazvVoa6GjWlpC3Mz7fRZiycgw5Nq4fWJiXRKbR0nUYoRJnp9Wj+hG4QaQdlUQsoaaI7N481ee655+yfL4xatZ7UhqEvMiJrR5/wFRXHKahTKlWfpoj+PCSGNBesu7dHh8sHOIdZP5aw/r4+bRYOwKc++XmrI8Kd8qL5TTfdFBbc5wBB/YtKA3h9X1lQR5hAgdlS9fxTOUk6pfyGdYNcHz2OvEoYiAaY52UD6rEgvY4WIs7m5Y5Y4nEv497ZzSgally3jEmt5DlzKmX9fUOSaHnqqafse7ffpWfDfwe881126KcO176OdNNISfWb8UNMGAioRJfQxNiIjW3dYt/97l02O1dUnffiSy9VZ4/wCKaz5/PKAbu62JxJ/RvyC+5ZXOq+PkVnkDMkSBBCZ1B5rrcQFDK4K6UjQbxBjQW0iBKtTU2FpoqEDQ0O2uT4RDst6+/vtSnVT71dDwNOvk00ghGgzZBGh8hdJtyV5yIlq1TtqquusY1btjgwxXiXzk67+OKL5QyY1xv7XKVlVnP6Y2fe97eoljVaKoOkU0itYh5//w9/ZOvXb3ZkO6DW+a6sfemLX7Levm7tEcn9CE12MM0bKraNo+G5eoupH9QIAkr5cTuGYvx54t6rT1So7EOjfAHFvcz5MGtHvJj76pYB3Vt+zmHmAfBhqqSQPwmZTSuUxDrr9UFMjAWkQO+slIoOC2WGnm7mzXpozWu+e+u9VqxQLvIcG5Qaa330cUdaR44aoHsyPodwiNwTj0sNjIkEg4OUn6DN+dgJXouxIc/m67zzLrBn//GKroND/oMf/EDXIoApCJe7JU0qf5a1C6oDHFxnS7EYgSBOe5tANi8NcB9x3WL+F8svbsx8IoTYVCHfUXmMhxoeGmkKX3pg8pQujIekajy4IMmICuB9Vp9LyOcHvX/xMvvG+ef67wcOefTwsV4vDrCZjY2N6v0mx7aIVLB27Y1Wrbm863nnn2/1pkcVsSdWWEgKI0uI1yHWFsZbpUTyQ6YFhFDYm098IBpeyimOHp6LeBGUMMnbMAYYAg4/h1czk8MIEQ938eaO+rqQvKOrGhpGDbhSUV1YDKka2ljz4qjznnGvnHLy6TZD6EnbZSplb/zXN9rhHz9cCPb8grdoclgKc3PtqQmkPzwbPc+sWq30rJUDlwDQEAJs2IUXXaLuNEeJHbR898H/x/bYYw/dWxh0IgfmIvnOVch1ODqtMlgoHUXHyWeKeRV42yoTxUkW4AA/vv40HVwv1nuNy7WCUGrfNjdIag4wi/CaGmhNw3E1CHr7DF2Va5Ipm5mb1aLNzc956EKY1dfbbufiQM3OM8LBgSRR/SgJ1Gr26ONP2LoNE1YLTfuiM5rZ/ge91d75rrcp+S9XFrRZevv6pWkVwwfCiojETk5O2tDQsCiOcDCx+Ljq559/xdZec5OzojJpO/PMM+0t+71V5QG1DYa8kzXx8ZGOMjt44iwf3q9dZhHAFLS6aPRG/IyJ8YwuDeTzapm82FvL0uHgAn6p40gHFAzUmzH0uRTbA9E/Ug3lNYPkKb9TZJJ809Uy2ZTcj9Q3Mx122dVX/X/qqzwvv+4QliXJp3P2wgsvyivNTI/bKy+9YNde+23xfTvyHXbOOeeoIcKHbfuoTJ4/B5c/RdmbR6DAPB1ijnC1IoMtFDuUv8AHCGWjvE3M310s1nNwiBaRaIBnivxdZiupdVIhposbaFIC/HKh0i6orxnFjYbKiKw/xgQnETuv4CMce+wJqihoHEjC7Jijj7HXv/71Mi5TM5MiXajxo8kAbHdUHNyobKIeayKnYtkG+7q0z0g5Nm3YaDffdIt15XtEBfY6f8OOO/5oH5fZpPfcjS+/42lZMHA5Fw2IXnR7YEoOY7upltsaDvyeEw/edLom0vNUeWgcRh5SpeYgFDdBmMvq4WFBxxYtWuzspECtw1I6WuZeyEsk3iBeXPDal8acNCBtw/0sW6HoPGIvMZS0gbjQdes22q9+80erUKZrJKxKY4JCtqyddfbp4tmqnzPwgBl1QdM1G4LWv4hww+jRjfO5INQoBtYrNj251c48a41VkNbs6LB3vvOd9uUvf8XQ5/Vaczg8gWYXrSHXuD3yF/NgSjryyGqccEK7AJVAT8N7VGtlARNqzIfJJaCFHCq0SsqaekikyQZi67hahg+q8rAX/EejOgFkJsfFn8XSX3zJFTY5MacOFkpGV1x7jVNRG4HrGmYUsWEIDZkRBELK88Iw8iypp6+5/Ep91g477GBHHXWUJGzdw2+n0ZzyziYMrufeNevr7bPxsTGV2DD6TlsMwFU6LU/IYRG4Qm0fWVUiGiKikJrJE0lTmbZMP+jkgLCylENnsoqaRke3yijy3FnnOC4Go8rokZg/I2DOvlAE0NVjR3/tWCvXvO2U91t9weq24By1e4wCXABq3KJqUnopLrSbIsQ6C5GKxuWEkPu2m79rr7zySpjc58+PMtOb3vpmr90DPtW3lfboN+ZecSzsUV5DM76GnGsfeVeUkzRcjCDiIE4KImopWuL+605qyVITIlc4wB5+IE7FQxMTRU3AziJxJoeLo8F44cN5KpAG+IBY4lHZgf7SojcnYzUV3nZ1e100gF8R/QVM8k00bb/89eM2OVmU/AudFa47lLCvf/2rQoMXL17i0wPZiEHrSXlXl4NTkZjNdYs5E8oWE+OjlmiV7fgTzrPZYkWh3YqVK+3yy9dYPhgO0Go+j+ti80Rks81cCSFLLF+ogyhI18a/c4oBkCJ3mZqsE8QJieGvIHRmVik6F9WNg3teR/C15GFwtkdBrpTh4SEHpjA5ZoXCjOqkd/3gR/bM35730Y8dWVtz7dWqxQauR2CseY0TA7l5yyZdmyRiBC6lbMvIiJ1z9rm6nje/6c32mc99Wt6Wnmc2itrN1CEWdLe0zgyy8kFvhbl5eV5+Z5aQlAMS5hypw6bsbCOMuLxlC0ZVT7uvNYJlvb39CpkRoQMzYM9QNqJ8hJGP4evGTRt1L+wnNbS0kK/13LFWQ9cpTuZzreKTTjpNooJcE597+RWXK0KQqkqomqhvJmA1Cl0hFgklJyWpKIoU040DVfcG+gvPv7Dd8+zD3lp21tlnW61eUkO/UPXgiSXXm9vGw+bCnJddUelRxqMEv6Gse4vpHPfP+/I92HqS8OXgikwgAGTbgOGFEghdWtaNeqF7gzC+IsD09FjyPW6I8gcfIP1gkcC9JQtJDh2AVktkdulM0UDd06XEH2OANSNfZWP193XZ1ol5+973fmKNZlKhK3U8NvPb/+1Ae+97D1Z+Se6LkvzwomF5D8Lazi7E3wBSumTxBdhElhIGoNaw8bF1du21t9vLG0cEbpEL3XHn92V82FyQDWKtDKOkDp3Q3xqNAmsRv+dKBXHiA43mDsqR15Jrce+cVh/9gZcFkeTjIBP4a7f/UggehMBleDRMzZUXiDrY9KxHvUg7Hn20DXvyL0/Zzx76jU8jTCbsyuuu0WhG16JzBQ82iCis1rLR0RF1WLGpyDG5TzbELbd8x1566WV52z332sNJFqE7is+ltkzTARsIYFEU1nCARfsLJSnm6cxMz6jDSnsmIs0IDII0Q/VUzXSb8kXctF5OyQqrcKTXpWR4koThfM+F45taX4BBPCvOQWmR69/rWlj70dExYzby6aef5dzwTEYp2iWXXqIDzz1KDxt1RdRJAoCqSCPhz1CrGDANX1GR/Oyf//yn3XH7nQFdb4gAc9BBB9p73vs+9TsQusOum5mdFEMs18mUQq84COOobxsMxxwnDBtGZXZuWpEb9yiFytDMT5sga4G4ROK+a7/egg/LFHHGR5JtoVAfmRxYd+QwY60MaJsF5IHHflz1m2qaHdaxYLWq53wc/GLVxc548EPDfSqao+bAgsVNUw6EAKkVZDI2OTlmjzz0R5ukKRwVgjINED4I6tRTT7RMh3t9lpB8EkOhnKNMWO9KGfkcxsQROlngUFeemZqwf/zjH3b7nQ/pCWNxb7zlZlk8MYkq9PXStVIVuX94eJErFtJ+RoknoIYxD8UgicqoRnifL0w/L8DN+vXrbeXKVQrTOejRIkdiS7nITFW/Rr54QP+vr1hHJ4SOh4nWwnq1ZPNTkzY9O21rr7pRJTJSiHPOP88Glixus4TwjKqpJh0sRI2QL+RKSQ8Iy7xs41QPDvj8/KyuDSOxZcsWb1ur1cMECBo9OmxuZla5JPeve04mnSSQg7nkHjWi5uSbEYQkdfGKgHsvohzWGw+4aHhYQgaEuqC4eN9tRtIUzipCCaCh6K40uLfQiMrLGUgFZWbWZqenlbsiLnDp5Vdp/TE2O6xcYcccf4wNiIo532a+8XzVNBIQfcpSNIggqgciiYpHviNnKIqyRtdde63WRg30zLhNJ2z1Bed7ZCVpHs9rOzOpNiLeaFRUfyZlIn/m7BD5lCrwsL3pIIUogbrfaO10FUhPZcNgbdoh773may1kPVAz8J7clEZNxB5QNsLkxIQWQECFKGVu+fk3C47FG59gqpmLuUHL48Hye9mgesfGIQfjcJJPefzuvFVChsmpKbXcMT0PdtE/nltnf3jyRc/VJHHqXucbZ52qh04k4DfX8sZ3NHXzOYXGW0e3Wi4LTxWqGGULF+vmYJYKBdsystmuWPtd1+LNZOzk00+xHVfsqFCPh8XCc10+bNlVPQh7hDzmaS30NrG4+QgV3Qv77BuF6qLRhQl2otlRH/ZZw95p5MoQymuCp/p/HVwPkx34wxGLoMEkvZq3zJWYElev2PnnX2a1io/M/MrXj7J93rBv8A0eDbDRoM2Nbh3VJEM+n4MLM8nbEL0VL/KNyad5VuSQk5MTPi1AFEpU9f3QdeUcDebvHCg8Fp+FJhKbkL3BgSeagxQzsmVE/160aFjPTCgw6RiIrAAwNI45wI6qE45u4+9iULy0xF7kOvEu1H5h3oEjMEYGQy55n9k5Ic3c49jYhN1wI8BbS4DboYcdZu/6D8Ta6GiiH9mbHdgLVDk4/D5NsiXPWpFcqzcTSKY3mRIwdd655wZCBAe+Zbvttbt95jOfFV4SU0D2yuT4mEvXUtJr1dWbrJp81gk/XoYEvHTtZv5kHbmvPM00AsYoU7oaqgz5fdce3apX2YQOJiCVUqnA8vDGZRY9AjAiRouQ4P1Er9ltd3v22We1+IRo/NxHS2QUIgA+8KV8L5HQgnR1d8nqR42dWMfDUqthvcoGX1BR++f/86TNFH0qu4crZq993Z526Mc+JiaJM6a8zolECRuPmySkW7J4sZeCFhyBFpCBNW2YpDAvu+JGWyj5Qn3ui5+3fV73Wh20vqDsEPNNrpP37+sbCF1CPk6D+/OSmDPLsKw8rBhKcai2jXJxkoI2YzikGAQYVarnBn3l+Of2xImItup16FYHWRzJ6lTKNj81pbEjay7/ltISNjVTDd79/ve2ZUw5zaw76wi4SJ2WNQEg8Sl+LlPD57Ou7im8UcA9QkXAIsaRkJpwm3vtyQMgEa35v2OpCnCKr8iv5fDDQIu1Sjaz571QZXkGPsRtYKDfe52Z3IixTXroyL1jGOJzlKEALESSNwBhQvxDnoih3mWnne2Vl1+W89i6dcxuv+MH6osmGrhszRrr6e/RffAsqQGr8yxwChRthV5q+MVk8gulgiKABsL1Xd32x8f/YD+6//5w/z6U+yz1L3fI+C9avNjxFgFoqGEWpN6CAin16VU7rLD5BW/KUDtoEBfUtI06Rtlr7ZhKjKaMYI/PupJ0zU+/fVqLmTBC4zro2ofHm9GAXt+I7iHYTKB6tGjRihfDHq/jegmJw+FcXuaUer21p2dAi6y2LRYGLeHAuGEzqCVLdL6WzRfmlQ9pYnqrYX944in7x/OjVmEqedpJHb293XbBxav13rOzMyK/C2TBK1a8yM2GIQTiMEUDgbVmU8c69Y03f8f+/txLlkx32P4HHmAHH/xu6+vvs54e96gYEl7L7/tA5pLrUwk1RioFQgnSn46eR+oaD2J7RJjr4Z7UtRIQ4TYVUt4UL+JhlXtfD4vcUIX+YCHLXprzdjYyE1oXG1YpFG12YtQe/MmD9qcnn1MueOA73m6f+txnFa65IcFD08XE8KtuMb1UzlmAwMBByYikQgcMz5CwlvQoKkZoh6UAACAASURBVC+SEkH/43rk+UM+SwgevRVejnyT/LEdjaj5o+agWda7feTFa1V58mjlWGO8L0aDOinhdyy38QxUMgztlLCgBKRqaDrcX+ezc5iV1kGlRXJWhq0ksPPvf3/OfvzAz6SAggG54OKLFFarYSD0BUtqKDSTKELo6ZH+tkcTC97ZQ5MDnq9ldv31N0qQn3Sq0qzbrnvsbh865FBbvGiRX7uqIR5xcT/cg6JUzUT26M3vAyVRE/9a1Ev0pQuz7dIqpU8MF3ltR2hukOe984pjxJwCmMp15W1gcFjaQXNsiNlZhTaEJdwIFgO9IW3UgBiSvHMBXJwslTZnXQ/K8ycHCbBmsLG4CBZLeWgexYox65E19noobJxicd7ynTnbsHGTPfAQM4MIq50yxvuffd43dD0YCRYAz0EzOGmvqHVwWRcKMjQAV4AvhOdszrkANjz6+B/tvvsfVqQxvHSRnXbqqaK+8X5sBJUGRM9DVBxpWK83O83PhdnxRHikeGij4oFCaU2x94ZorCehspPMPeRct26dyi4R8nedLydH+rQ/jzAUVYjh4oSKgLuAWklxEw8wsXWL/f3pv9kdd93vSoL/8i92/MknesN7kkhnQSUdWE0YEAyOG2gOoYumYzGGBwd0aPk5fFueLZ8PgwyDhSdRKae9ocu2bNkyeXEOH69nraenprVmPGcOJNEFBkM0UhH3TfuBCfQYWW/hc2mdhbl5pV4idiDVO+PyLjxfZv8op+WAhusA12ChlE8H3jKLRW7KYRgfH7UHH3zYnnn2eWu0UgK9zr/oQoGp0VBCc/Qw3eWLMKZCxRnNku+y6ZlJIcystcA45FcvXRP6fVMqWR59/LG2eNlynR2+aPTwqMCxE0Jw1aMR7gspBevhDqDiUxOC6gc1a0lEaY4VHG+X9eV3wZCkvf3zOy9poWTAg+zuZS4M9bmqjY2O2+v33VcbbOmSZWHkxBIdZh5Q9DRelHdVAw5jLJ+4En/C6kb4hYQHC+IFfTFjas5jjTKm8sLE9QxXatRsfnbGCsVZe/yPz9qLL48GnVk6+ZK2/4FvtcMOO0xIHTKX6EvR4UHIw0bFiMzMTNnwokUKUdTMQFRAaJdyZHWusGBnnEljdcv+5fX72Be+8Dnr7emVdQUQEQIMUt2ZVyTA1D02NS10WOfIueWQIsWC9RaIIhX9jIwGQEcElraFwV5bFaQfDmhUN9jmdd3jKpwObYV6n6DOoVxTSKvXhefmpm39Sy/ZFWvWqmtqaOliu+iSS7xnNXhcnDYGLl63No8+wxs3+OyB3h5dGznm1hFyYZPR5sACsoEroBtNWI3UC903ArDKJeWwXsP3ZnCF0t09WnvYSbGOT2TE+5B78j0+FwPGSBNQaLI+RNWef/55HUZVPIJUjdaX0D6R1IHGEHPgqDDgxeLEB7w5DqBaKdmG9evUPLFhEyyxhO3xmtfYV486UjVxDDPPyidUeHSj/aJ2vZR1hjY79gRccgTvuL+nnnzSHv39Y1p9bB4O7+TTT9VQcVoNcXC0xHqjjosvSISePxs1vQfeevkOy329lf54aZCcXcYyGCcL9EvO0sycI+g4ocTd153WciZMTioKkCLwZIRBLKZD1ynp5bJBPY91hDDX0eVNBrS4gSTyPbwNYWtot+vu69Wh4X1HxyfaKhiUYQiZgMyxfj29PbJWqO17aapm83MTesB33/ubdkkEz8WDP/e8sx1NTPiB4XdYJEI1RlosX7bMNm7aJMALhQi+6MFkqgB/0lj99NPP6KDv+/rX+USDLMp83TY3O6frrahTo0fhEfTHWAYiJ+MACGCq1rVhooavuocqVX2PA+8lrj43dIEhFi09axQNnyPOHh6367ihruu58fajM32TRaQREGdkdL2dc/aFyqcGh4bs4osusmTG5yU5m6elzc51xQYB9cuqVu2gGpxh8AeBlJq106VNRWkHz8i6cj/i0Qq0c7I94anWX3IwKRkCn0CfkaFns4k1FFBrDvusWuW8g4fmj5WrVskQ4+mXLl2qw6Mp8Gzmri5J0PL+XpGAI0AImbGZkJ+yRgpLg+wMnHPC6S2b19uN199ko+Mzlkhl7OD3HGyHfvRQa9B2SQlIE/e2TWpk34lKSQoHSYTcWuW9ps3NzOi6rrvmW5JaUqkrmbQTTjzB+iBTwGnPgrJ7js6e4F5UbQpG2IFCJvwBotV0b6Nbt8pB8Jooy6soJCDnRDviXTcaqm+zfomf3HZhi2Qez4GahLOjGCkYpu9Rv2V8paBqs6VLlkpAm79X6VlVztohDwOXVA3QeLS5eW3KVTvvpA8Tb7fpJQJCy9l5FDOcUCA9KknB+phFrCULB3+22Sjb9+96yCamPETnogFaPvXJTyjsmZqdbOfXbChH/5LqDIphFtgWjfcMOKZvk02KMr7LdHpLIA/He3H53S73sl09CsM4sPCvuW5a77zX1GF8BmMBiBFCDQzQ5gVwBed2Wn+Xoh8i2v39MkwAMOqL1ZDqzYoKVNjaLjzmgQlIUwdbrBNvk+l0rnGYsEhIXuf6ynbiCSfrcLEZ1q5lHMm2nmoZHTMBdzFiYB0kM9rtE+5A7oiGqNFiMCmXsN4ukOdi9BxoSmSvrntV9FMOD9dDvsyBJ58FB/EWNG86YJPyPKge8EyEnNar+j4HkfQrln2oZvh11drlJF27DrDLFMWUjIOe0cR5fx4R6FODA9GeiB5NO/HkkzTzN9PRYUcdeaTttNNO1tPX3R4Y7kqOrrAiyaTApKKGzhfrRUhOjXfzpk1215136TPpu013dtipp51m3QFJFkmkUhZar30TniPfJ3Xk2jXcjH+Des95rZ9zgKFiD3leDUCFk4K1GAbOC/Nwud3EA3dcJsojJxpuKDeAu0cWJOorp3KO+gmc0OCshHR1N27a0EZVyXFiWURsF3ltzyPwOIrnO+kzdI1eNTGEw0CeGRHJUpEDX7Mli4Zt84YRm5vdauOTs3bvvT9tP5xyuWp7772nHfaxw6ze9HoX/7FZCMuY4aoQE5YLigK1mnIxQDVm4fJvroNNBljGgWKxObBYOsIn1mNqhnqnayBJlLVWdyudzcmy4528tIO0aFZIdjx05Hnx4OKxly9f7p0mvB8Qf6BJ4pkIaeOsIG0+SeU43zcizK7cEL2ue1yMppfEvM3x0ssusWee/psNDw3bBRdeoNEVPDM3TOT/EPKZ7+O90GwqNjk/5PPTGTSavEykdchkbNPGTWp/5N7F2ir7xDoaBRSoi+hPf+yCDCoblmdPuqJul1Dj5hoAHbkeqJSF+TmRX1DHEPIaJkIQwRA5DQ8NCXhcvwH5UydOyFtlMup5Rs2T0JW1wuMT9vLzKOYAAozXQ9HigQcfsod+9ogM2qXf/KbLBNHvHO5ftfgwHV5chihC13R2mdawUbPpiUn79a9/bU//9W86H6z7hz9+qO3z2n3UZonDmhifCCG+r4sojxIYNI8GUQOhsSaodWjPMsKFXJq6c9DOis8+8ptFxAjMN13T3TevbmGtWCQW2vOJpoYUUfei5zXWkLiQqMHEQYSooIG+hK+0e6E5FVrAfMM0BSpA8BfPMnRBKLw2J4uzkbwe6nImWFAWESs0PTlhhblZK5Xm7bbb7rZKVfibVSo+OOsb3zhFdDwOaxQJw5qh37NkyVJHYTmkUTS7s9PDopBfOs3QD4NvXJ8WoMHeoS2O16vUoc4npEUyolYuFLGq3eoBFlraiSbTVtt9993VZM3G5UHwXhxOQs04yYADDW1TTRvULSs++TxeBwupxoXwwD1UJix1EXGiCnFnw5BoQDmMAtfOPbMx5a3D+BR+l++DTQCm0c5HLZV1Fxm/XcpquTHNuNfAC3JPIKWkHfybe6F5RCWJhBNhAFjEpAp1fg4kkQLrRkjLwfJIzCVvMBpEVj4LykeaqM85iBQqrcFwpJl052QYPoP8j+hN0R1zkZnDCzc6TLHHywoQE6vLa+UxR/aupAFhHOL6Jj2i9CgO0NEb1ON+EFspUHxZ73Jx3sZHJ+y7tzDNsKa1xSmccc5ZTv1U77VfZ+TCtWceg8oXCsr52UfqE9cUBFck4SC7Z3eBAHJ9DjYRC5x+rivyHhwHSVjiobvWtBgx6Vxkkmum0TWtkWhaZ65blpzFcGU/V8b3oUyIwvnsl7gQ0VuACBLqxFY9vPHM9LQsBt6GUDbb6eUUwh82EhcDOIQV5RB70/SCWtnoQnns8T/ZY394UkbEZ+Sm7MijjrDBoX4hdlh5HpZ6cxeg5rkFhjiBtYttW5EYTwjiuV9TVpVwn993BL03jNx0obFYp4RiSU9qXz96TS3lwrvtsbcOHR5WZZX+Pv2dz8SzsSasnTwmn1XzLpdVK1c6zTJwwHmAnuN67qoHRT4emGF8H91o7pPnAT4FRsD6z0xPel4ZIifPxXXc9Z6RfgrggVHEuCl/DZJDft39ogyKg02ZLvT9ToyPO5NIw5l9jIlyZJWTvJbKs2PzQaLh/VkDMaVk/NEYg0SQtgWV6FwelYMbc9Kx0VE5Dg6gpjdQmhTYWdckO3jU3DMeSyIMoP5SHWFmL9ex4OXHUGbhPRj+xvvEBhb2AmBoVJFgrahJO4EIMNJJ/eyL2C+LjpYbcP6vZi88/7L94Pt3qwIDR/6d//7vUgrxBhQOPVx+LyG5fDBytB5NxsgEOi1ALfsUI8nzi62ArHPkLHjakdbBxYjLS4f2V3ETCJVFPVOZxiVDlDMglVEs29DwYhvoHxRQ5cBEXhuG36EkRElk8eJFNiutWQcmWGSsI9aHkEYxOpZNbW8UkskvPPTBU+G1hUiHkYtxRg5Op1YuStFw3boNdv0Nt/iUd7G8Grb33rvbRz7yIb2/K/y5BUces1Aq6SG47AfKBt7xoQNLaBg6PVgMrtfRPY82+LtI5gAUoJa8V2fegZaBfk2B33XX3RQ2Tk3PCQySqBh0R4TGOjoEtmGQeChqN6tV1UWjqXP5vELNZ/72jHKZAw84UPegUDp4WylKkJMuLOi9d9xhB3l6CWnLmHhxHw9EM3zMg2K5iAcvFYlgnOJ98dxceSSmF5R+fKbt1PSEDrBqp8H7gETHLi5ycn4WW+AmJpiRO+RhNyywUKfGQzt1Mi0j6sQJBqF7PzHOAQQboIe1IqfdsGGD6I6sNXk/e2l+jqnvPhGANaDUFBsTiB4wPvGQz8/OKn9nXQX8BPJDYX7WwUPCZnAJOtF6eqwz12VbtgC+dqiZgc/j4PBzR++JLd248FVr1tTNdc7Z51kuS9NMwk77xhmWD2NGNGm+XlW6QN6q2Ukq73hzSCz7EYGgPY3zIv/n/tgPrFVspMfAqhRJpBRok3HvRr584kffu6yl0EXuOKML5hdgTnnu0KlGcw+38AqxgIzndC4mm4nQNr4P1mjRcCjF0PkfSNKx3snDQic5ItSEztyItxB6Us8NYZHYaAAuszMT9thjf7Bnnn4xdNI0RXE85fQTdYB4LxElFD7lrVh2Jg8v5nuIgvHwo1wOOTq1Xg8LfTQGm4tQ0nMl18OKXi+WTJRnZbPW09tnS5cst3Taa71bR0asp5/m7U5xlMmXyWy4Hx18wLLpGUH66vrIeWSAl1g0vEQlBUJRSQBpyIELsRNBM+aRtePhY4Q44MuXLW+XimZmp2XdOS3IikbVB5rGly1dai+++FJIKZhQx3QDrw1ivHRdMzNyy0ReAuXI18TbriospguM73GIQUmdUFO3gaFh27R5cyj7lLUPCGPj3CCfUuDaWy6iwExbryQAYIk1lUqqbs+9EplheOMeoPWPgyDEP5AyOEQYNcJhSRmFEk4k4uAE5DWpPde2TUXwkR5uuB3xzqkzCU8moCkSPJQmecSDSotmBYEnbBedUY3AmOy7776qj8f97Q0S6GA5b53rJudXX3Ag17A/XEklODmGdisF9W4wIpioxhFHjjhD0NMYnAlGIfGTO9fo4HJx3d1O78NS7LXn3vb8Cy/oge6wYpVYSngvXudzQJFc8Q6N+MEsLl/Qvcjv1LIU3o/F4CZk9aQ36zqxWCfek4VAw9fbmpyxFRX7CbXGx7bahvXr7ft3/lAaQlEB4evHHBXC4G7p82DRmE5OO5rCRw3faijnJcSL4SgbSXB+AHxY8CgSzsPn2tuatlGdMqh3gE4K/at5SEoIjbUXEIaIdtWjDv6LFpjPldxL0eVNRbHLddjmzVukErF8xY7aLNpMKEKE+jDX5F7B0Wz+zXpxSLhHDgossfiFCke0ypk0RsjRejYGUYd714ZyWIw1hjmG2Zo+MDCgtIEDTJjHsxDxXjUNJgV4OZDfLWqcqOsBA0Byb3wW6ChGgGtWjZRDgAcNhA48KgPbuA+tSSibOTjjmtwcYkTiXL+Mg+sbXDgAZSd1yczLK0rOt97QgQc3wdBzTzDhRIhI+GxaB5kQ6+/TKBLXE4tSMj6GlahQTkpcdMLcbc0RGB7Wjb0TcQOF0YFJxnPaHvCKZdLI6WfdYq3Pwc1SEJh3iSYdSPjQ0qqecVVNgW7cs5f0MEhCzR+860qhyiwKibv3vjKR28EPFp2DouFJRW9aj83vxP3KS4JiIIuANaSlTAJe0tXJtlvwonypfr/sdVEOKEgvB3ZoyBuL8XYuadKlG2GTzk5PaF7tj3/0sG3ZPBbqmGY777arfeLwwxXaU0cjFOfArVy5wjZsWK9Nz6FsAzZBYDqCZzzVqE9E2KoNWSyqiM5hZD0wHJLHIT+kuVoHOWGLFy1ViyH5Oxt+enZGeTqenPVkU4Im8wBZDyHdDdMDIb9y8GdE2lE77bqL6nkCVBLu1UFcIyuJa8IgRuSe94ujKXffbTd75dVX9bO48dXAX3HJVw4qa07aIo5w1TefRlqG8TNCzK0lMgThN0Z03br1Xr5iHAeT6oLgQQxdKzUIFA44Ue7ivdjYTmllH/kAa/YQeABGZK+99lLoSu1206bNttPOOwmEZG3Gx0Z10GNr5NLFi9spSFdPj6IRIhUiQYnei/bqbYkC7wK6z3uLRgn9NnQPRa9KAz7eGULN7KzvUT+8pAwdGvki2iRRaMajnGiQKOdg/FlDdSjh7cVDQD+cUlVJRhtjvXnzqK1cuTJQOSHpIEAxrOuNnykuROhVdnEAxoQ6YwyHE3W7uGfSCowv16gJgb+8/4YW4QCHgxonb4Rbh7/sOkD9No/anEYzFGzVyh1tdsZnp9CRwYIhrk1xmvchNCMEpMYWSQexw2Nqerpd3iCfYXH4fTY+D165cbeTGTAQgDx4CGiKauFutmzdulftttvucBCnRY9qhx1/8klqII+80wjD8x4Io0dubkQ9IwiBd+MhRBTVhejo/3UpUg1xDjNq2HRxTi6bVSGX6tg+uY3rQL9Xqn/kcINDAmswALxGiGc2o8OD1+JgIYvD/XPoXrvPaxXV8FpFMEGtYnJqQvcVw2hCcA4HXVQ8bCw4+S/q+9G74X0U7klQzdVFuKb43soP83ldM3+PKUZPb5cT+pFuEartSK84y4FPrWpCt0/Ac8wjpDZdcNgn9Yzo2WXTxUPFvbJxd911dxuiHFepSO+K+q16W2HepQEG5wOg6e2RFP4j7ZG1IzReuWKlHAHvzT6VMlGYmAgOgdGMaDH/pv6u2VdxhCXRkLrbnCQSw1KtF+iwaKeek1Ka4nDJmAZhAO4PcIn8Wg6ICEo9x3hoz42JbMi11WJIWhiINxxMqix8eQTgiDZRCgdWbYQouYSxrDHXJvVRjblU0rlQBPXgXWs17JEfMmaDw0bdjgiSjckCLlqyRHmbtGeDcgULNzDg4SgL19MFAr0tN+OwKZfr7DSQSQ1SCiUPLG5nR05yJ5ETDMghS5JMS5+KjQ4QRrsgpG7lK3i+uXm77rrrbXYWhUGsedIOPfzjEvCW6DYHIoxu8PCfMNbHo/BweN+h4WFZbLeqHpoJYg9av5QuhCAX5uW9o6aUPGYYQA1pgXo03hgQig0/NDiszxCPWTNnMj5oOekcWWp47Y3AxMICD6JPv0+3kbScQyfPyJYtHq6LMeRDwvldlRSE+Pq/QUoxMG394qBqyIPm9zTLdnBQFhsSjUJfGSMvufAesSTV1+dT5CIUHRlw7A1KGD5Hx6fIybsDGs3O2dDwkM3NOrWU9+rp7fayYhN5Xu8K4lDw+0QNdOzgtdk7pA2sobqOJNnje5D1YCPLcBRLEmEgyuAZq2MLKSBCaqiFAQvBAPMzyCGUsYh+hhYt0s+5T/SkWb84PsSBwKbjECE9QpdK3lsaXdt0sajju2SS66ppRE44fHymIkzhDN4pxl5irSgDqsOuCX3WAau4jvw75tMKuSW4j8P0hvnwIByFl0H3MTgY5sRDP7i6hfWQNEkYzSE91xQ1NBdmLgdVR8KJHMoSaBgpHNqmESw1Wak0kB/5IKyYL0dPR/4QifiIzmFR2ORYEc89E6Ii8n3AF7yTwnb6GFWg9+6O9es22g033KiDy3Xstuce9qFDPqJDyesxJEIc1e/bLdYLv4vnhfmF5cMo4AWwum4pPWRSGCMFyW41PwvoYWg2k+rVweG9sRGaj3kb90hfaewI0XCpICbg1txRXB7qDkxKn5wUQo4n5GHKC4f6Kd7HqY88yEIbrYWUwOt5ba1GiOraw2xijMhee+8VaIJ0L3W258KqZS6Q3rlu5U9C3D2EjnnqwoJ3VLHhhgcHReoXaJn0/JTckL9v2rxJhwKjBm7B8xobnQhlvLyaNYi4IjhFXVec5Q5+5iAi98hhxejwM0UGAJzq06WcBxMqKfaW5GOQPgpD1+ANq8QVOMbq2qrVbXxivL1vqFZgOGhIUCkmcAqkpIEqxbR3v3H/S5a6QDkHgrlUQoMVBi+0CUYQhiKRBWejkmkcQK7JGa61jcHnekhz+LmrdlAtIAXyPNq7rIhgQZgH5ElVsgyCfP5zb1mNgC5nkjIlLlZ740d3rRWtQ+1wuS7beeedVfoZWjSsXIcL2mGH5QGE8lYpYnh1uaBYqLEPxOqeF7CAeEM+VCFVyXMCHfSG10yxtj5P1DWN8N5sNDYNrB/EswA7IDJQVuGiG1JzNL0nr6c7o1Bgoh+AQtbO+MYZIrqLtSUVDpBP71DR4jFZjsgAiRwAjyCu7rQ838hCtfPdCpVFZEDnCKUHmrYVevqBEmAQh35r4rlHJhIfQENYAu2ICvjDVWjOjJsGEj3eVifBsKAjrNqpwAlv0GdTC6lX3ZgGBxcOJ8Tj/nzQ1oz+zfswo5XrwZsJIBGxH86413H5TIgo5HYoNsS8LZZ9eE3cILxvDKnVgkcXF/cS7hFjEUE/nAI1WIwk1xvzY1InDoL6o1MeNRBOUm9n40oNEo9a8vk/UeKHtcX78W/xAIICKN+X5GqvixJiANmv/eIf0KGVs+npMBKF0SYFat2wAEuaOhDJPSDYqslLnZS+VkaXIL/TbHPlNYw9MLCoHEiONVQSeD93DC6JxLPCeVHFYE3c+Xj/bDrp2loe+XjXlzqFqLA0mzJSNLrwjIXgy3i7cCLVEkWPqFVmaOlzuVmBjkEuKvHLB2+R4A6bhXsBIMITkRuwkVhIwjLfbJ1SAwC5w7tJTKtUbBPzuSlp4LYSYhXFRgNyMg5k9KocRAe1PJ/i4rE6nrT78CbAEfIVvg/ZgfIU3tNDu5r97OGf22//91HrQHIllbArrrxKVpmNKzkSych4aB05tHgnrCpGBoOiujGjKygvhEK3y6Z6mYTP8oVPKa9nLbztzj0714HCh4d4zmwSQ4YGAwmm+b1E7xb7TGMvLNeJ9Wajq1QRuLh4FvIcrsU3LTK3PodJXNhSSd4KY8drXQYXxpnTL32WLlGE58saZyn03NUjMURisqWZBtEVpIjmJEbA+hMBqbc1tEy64FnSmXIqw3h+jXAbeSnXHUdv8nPqvoTD3mTviv+xOYBoTTKooUnC8zwP+1U7DyguOTTeFnIPa+NtkhhJclTPodk33BBRCOg6ObaDe3QU1WS8aN8B5+AzyIcxBtKRAmkuV6T0GLEWFhjPiuHmnoeGFjkmQVQSJivKgIeZPy5BhFekf91VXSI4mWx5muYgYsL7xoOqpXdlIcjrdWM8qWYFB/4An+FVAxp0vOEj7jHuT/nxQ/ddL7E4z0e7xOkdGxu3WsOJ2yIwQE0MdDo+Tq9PJsRo0thCrAxhRo55sj4NnA3FwWEB8b54Bw4zG4mDy8YUZznr8iLcdERteS/4qBw0DozXZZ0YEnPVjRs326233i7k9JjjjrVddtlVjeNC5BAOr1fbmyl2qAA++ThFZ1nxYGP5ieuIvN/22Azau4LeMg8ecA1LiYohm5V71EYMetLx4Ea1CZVUAuvMx3e4mrD3ETPn1g0J60kTOgc41lEVSqK0wcMLYlAYMgwe+RiHjlyIPx008zICmxEPhFHU7FhULTTp3SsHkSnkNUyPZvh81oH1xVizB+L0PDWHMMAKemAq6XOLNMmgU5I2KtWNjyvSYLOxyblXZxOlbMuWrerUIvrBA0stRU0DaJI5zZAv1oTDzwaPVY5i2BdqGYRFFsp9tMPhXFTTDFPsYmTDtXmNtyED5IJ0/t5DADtoVhtig56i8bkcGtZIrZkBp2GfsK54eYXqQfVF7LpZF4Gjvc6li51Drbp0ULFs1pqqKAiwQygiGHAZIZyPKMNet5ZHDdROno83y4Qh5DRjhDWKfdPKoX96zzWt6HUAZXbccUcb2Tqi0JTNIIQxlWz3XjLyA2CGDqKF4pysOUAPelIuPpYSUBU5n4wSwUqSH/T2+CK0lQdCH6iG+DYa2qSEyVE931vtAHdQcHBBMy92t5x9AxId6m5sLLV0wX2t1qT4wKaK6vn8HpswCrv7FDQPPWMdWy1dMLNc9E/DpllUQhgOY+Qts/h4bTa99KBD0ZwSmvjWGtTkuk78G29AOAuiypsARsVGc1BJDAgglk809IZuNj2bAiPjh5v8qEMgDcCLG9WGjElku4iGlAAABCRJREFUHLkAuAOCfPEMYo/00CDtmgsqW6E7heFRvbzF5s+rrEGP7Z577hk4z82gPwUN1u9TG0rDnV1vC8EC38hzWicOBJES3lLtckQIGRc6wGPCGHIUviBjHIEZ1p/35plyT55z+8wmx1JI0SDZZJ1LHTqzWF/RalvNNjEEZxD5zUSJpD7kwp6COKkldhdFAAjsAqOAB6fCwXrwGsqjXBdeE2A1aoJTHpXWVRgMx30IeAq4DYeUZxpZXdS1Fa1pjlVZxoQoTPsj7EsYdZLMRaww39XGROJ0DHCMOOlCketvH/quDi5vitQpC7t1ZKs2VqzR0sdIvsfDQrGdiyT/heaIM1CPJ8RtwBRCX+b3dNMSZ2pWANRyDm5SHov3jaJx5DtsClfLiKJrPkSMDaiQubAgYbeIytH4oOFJ2w2X8gHEAC/T4X2cYeJe3bVs1RQQCtqE+NLUCg8yymCqplz0MDpuEq6L0hSHlUNMjiTygggGSK24hCgbS/U2Sb26zjSGI67X0mXL9H1J0kr42r0NuIAMAZpcMnquWQyAETm/fJ+p6q5i6WU0hY9hDWJrIjZE94JiBV40IK4uyObPis/HoLjXHNc6iElWWNDrBdIlgkZX8BARVCRS4Nrd27nqSYyEmNTI+4JLKH+UtIxPvZDHWzTsQGMwyBHg4/f5OWGyWFuBcBCVDsWTDmJ/3D+godD08F4YONoo8fQu8ufKGbyXUsCQa1ZDjdm7pHwNJRUj3r3rb0e+tOeSTq4gxdH0yNCdBHYgrAE1yaCGKU4yfduhm4jzQmUF58L94d2JcjylcoFAOZogX4tmG/tAEj9MhdBEDAeAo5H2PdzlQnaP/eKOFofHSxcuw8ILyJvk7eBapn1GEMVyFCAJpTX/pVbWJlfTr3RnAy+YDRAI77CMsHxCfFM+uJeNF9viVOLo7fG2qqSDEIAFHAoWVaADjQ1dPdoIKpHUnZIWPRNWnwdFQo/VxJjMzdH0H8XcHBRjcxNe6nfDOA8PXbzkozpynkZ6R1Mlxr7dRAMvo3iow/vBPeazI9UzDiMTN3e7vC0CRmIJBfqjxAoS8KN9GBjvx4Fg8xEGUq/F8OEJvdifkPdQTTWQBoRkS8PJSxO8P/VRwMRRGq41+DuntVdOzGiZMJOHDeKAYU20RaIdZzT55uKwSQo1oL9+nWnV2+O+KFeK8q5qpaTPFK1r5u+EEFe17c5uB4OIiOgiChK6sfwTh8Lx3jxD1/XyWbWUsYg08Oisgat3NCSBxHvHvJjXy6BovCtRlbf04RBE+glD0/g7835cAgc8Jsw9qjnlF1AxVkD4GSArnpUDRB0XY6TSHNTgJFxjIifmCnmDCsqP8fBHYJFnuXLFCj+ImYwOL85DVMjQiKN6MEO0Z+eUQjr0FWq3lZKrcbAuoRWQn/1fbh9VCp+xIjgAAAAASUVORK5CYII=">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -647,7 +680,13 @@
     <xdr:ext cx="304800" cy="304800"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="18" name="AutoShape 8" descr="data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAH4AAACpCAYAAADtGIkfAAAgAElEQVR4Xoy9B5xkZZU+/NxbuarzdE9ghmECQ85REBQURER0EcOiIobVNbCGxV1Zlb9gWHPcNaC7ZteAeV0TuigrigTJGSaHzqm64q177/d7nvO+1TXjhq+VX/d0V9269z3vSc95znmDeM8v0iBXBPIFdLIV5MpHQl9paN//l6+p6Qn84qYb8fh0C/ONCHESIE6AqN1BHMdot9tI2hHSJMHfvuBsTE9PYcOGQxBkAoRpVt8DAGEYIpfLIo4TRFEbaQoEQaD/0jTVf/yZX9lsBplMFu12S6/zd2l/D9BqNTE0NKT3RFEH/HUripDJZPQzX5MkMVqtNjKZUNfgNYMgRBxFyOfzem8ul0MnjpDV++xT2lEbhXxePydJ0l2ZJOH92bWrCwsYHBxEgtieIYXWIghD7NyxA+vWrdP7/LNpqZEgRYQw5WcFuq+7H92JL/7oN4iRQavdRJQESHkdvp43zXtAqPsIwoz9Lg20hvy8OE3sd0kHnVYdmRR4/TlrsGHzIShmQwSd3T9Lg3wJcaEfmf71CDH8/1vwSGPc9F+/wV1b92GiGqERUeApkjhFq9XSwqdRB5kwwNUveZoWh/cSRTEenmjhqIMKKOQLXaF4IXMhuRm8wCmYTifWElEI2awJXgtoa6DXc9GiKNLfC4WCNh5/1+509Bn+q9PpIAxto/jP4PspeL6Oi1kqlbRBHn74IQwODWHVylW6Lu+hdyPaz3avS0tVlApF/RxmA91Txv2N10y4iXs2DBckoYJELQk+ifgwKTpJipmFRWzdtRdxkMFCE/jDn+7DUjOVUP3GS4MM78Z9PpAm/HsCrh+3kjYcYsSthhTwjecdjPUb16GUzyFo7fx5GlQGkR1ZiQSjyCQVJNSKNEQm5NI0uL1thdMiEPI7F8BWvV6r4ds//TkeH6+hHrURdfiB1LZI/4UIkEljvPXF5yFjSotWs45H907hsINWI05iLTQXmQu2YsUKUDBczGazgUKhqAWnJdDu5mJJw/zC2kW9heDDNptNXWdpaUmay/fZxuB/QCehZYm618tns3p/o9FAuVzWzybkRNeQ5gQBqtUq5mZntaEP3XIo+vv69DfejwkgQODuLUk67r6cNtIGJAnSBJifn9dreW96T5ggE4bI5mzT8TPnFmt4+PHtKA8MYs/EHAJa5CTA7Xc/iKUm7UkHtJeUU5gmiCmrGIhiW0d+ju4rTZC0KcMUf/XkMRx+xCbk+drFvb9Pk2I/qs0YhTiDXHMJmaSJfK6KrKxHKjMVZFPE5RFkBs+QMJfVLcUvf30jbn1sHLO1lsx9p5NIeFqUToww6eDvXnweb1M3045byCY5IJcijrzJ5AImKBaLWlgKkAvDf/dqqjf5XtDalE7j+Z2fy+sMDAxIUDTdFDq3MDfP0lJNz5TPF2SVKGhqJc0rtYXfqfVmIRJtBm+WeV95aovbQP5e+Ll8favdRl5uqI1s1txDQK2UVTBLwbXhpvPmWvcWxLrHMEy10WdmZvD49p1otGNkiyXsGp9F3GohXwTma21Umxk8+NhWtOIYowPDWDM6gHse2wagiKhjG5pOkMrEfyNqydS//IxRHH3sYcjRDV3zgY+klUoFU1NTyKQBchmglC9goD+LF55/LIbzixJ8JsigU8gju/J8hCltdtC1s61OHf/ybzdgz3yMatsEyC9qHn/OJAmuvuxp2Ll3L7Zt3YrNmzfioDVrzBXQLIY0uSZe+vp220wuzTW/+Jo4AIpJqof1LoEbI5PLaYNMTU3KHVTKJUTtSIKnkVpcXESYzWgD+c1CM9hstmTJKHh/v7wHCl4mmsIPAyzMzyPP+wiARqOJUqko7XdbH7EzqYVsQZvOW7Ukjc2sh1kkaYIwzwfMShHA2CPNIU4jPV8my+vxirYpOnGMhx57FAky+nwa93VrViMMUuwen8DCUoRCuSLXOr57CusPGcbCUoIbb3scsbM0iUx+jDjifXTQhyVcevpBOP7YI5Cjdfra93+cTk5OIZvPYXF2Dq1WHZ1mC83aEi668Ew8ZRMvkKATtVBZuw6obAJwsAu2nLTSGD//9S9x1+PjmKjTZ1mA4bUvm6b4+xedi3sffACDAwOYm52RgLm7qZGjoysUsMnP0i8FAbgZzbS7YCbsIBMtIc1YDOKDuXyxoJ/r9Tqq1UWUSyXEHXMfaWwWhM9GQVNb+RkdBXctFPMFZw32DyYtwMogl8mgVltCJpuRsKn9vGfeEy0X/TEFz/9nwxw6nagr+JSCp6Zn6EZChNkYxSjB1h/+AgPnn4MiN5CWzwJDfiaFVqvVkM/lUGs3MTs7q/UqlQoI6Q6RYseOPRgaGcHs4iJ27NiNeq2N4VWjCKI2vvrLe+UAJHSa+JhrEKPTbmEk38alpx2E4449HJk0QfCOD34kzYQZNFtNLRhVr6+QRy7I4PynHI/jBsaRBDk020sY3rQZcaUf2cxJ7qadEQ5Mw7/89e/gvskFNNsddCLz9RRAFhHeetkzcMedt6Ovrw+7duzEMcccI+HXanUJmQLx36npWgi3CWgRGlOPopx+G8mKd7hg0KL+TC4rTeQmu+22P+KUk09BTjEBfawFiabRAcplBmyJgj0KfqBc0bVCxg30i4r/GEMkev4AKVrtlhbcgsUIWZnkEI12w3Q0yaGDBKWcuRMf/EnwykKyCOlKqNWdNh79yBew+nUv12sz2by0ks/HTfOlL/4Lzj77LKxcOYpyJY9cJq+sIuq0XWzEOCdFua+CyalJHLJ2LRYbEXbu2YeJyVk8vGMav3lwL8K4DoQ5cylUgqiDVaU2XnTWRmzZvB6gqX/Lu96tfddxfpVBRtxsYMuG9TjkkEOwAtM47pAYzVaKVUccDpQqCDIbkIYruhE1nODrrSo+8cUfYu98FREFrwAjQSGu400vfibuvudupTrc0f19/RI0NZWawZ0+NjaKYrHkAjgL5LiQXPBcPo9Mu4qwOOjMv5QQoYvwd+zYidnZGQwPDWPzpk363Hq9oVSNLoAmPJfLY/v2bZhfXER/fz+2bNxk6ZpiAKDdifDJb/wSrX33YsXgEAYH+7VBR8dGkQYBRkZG5AYp+HZswhifGUchl8FAedRlCpa5cHEVIHJzcrMkKZoZoDYxhU6mgAwySNKONhQ3CTfiXXfejqOOOlKbJJ/PoL/Sp+C31WxZzBGYBeOO4vfFhSrmag1MTM4pGJycmMSP/vgomkwL40Qug66FmdWmkSxedPZGrD94NeK4jeA1V70t7fo4mp2UMVeMSy65CFOT0+jEAR579HE866zNOOWofgSFQYSVAoLcJgTpMJIgRqCcn0Jq45Zbb8cPb74X1VaLKaQWYTDTxute+EzUmnVF6ktVi7Z37NiBww8/HIWCBWC9QqcGc+GoEbx2LhMqIOPvvannxmCEzvu/7757sbhYVZ59+mmn6TWNVltWI+lESs8ovPvvu0+awLs9+sgjZL658crlCh7cuQ8f/Pb9uPJpwxgaGMTu3bt0X6vXrMGGTRtldnPZnEy/rpsk+PUTX8KmwnOwbk0/skFemRAjfL6v2WigzRRRAVyAb/3bN7B+06FoNprIFYq63pFHHYn60pI28ezsJFaMjiBIEzA2NHdYQLvTRtzpoES3FobIZ/Nah4WFRSzUm3j0iZ2oVhuoN5r4/UO7MbOUIHJ5fNrpIG5GOPfoEZx34joMDw8giSMEL3/jW1Lmf0p5GNgAGKoU8IJLn4PFhTrjEH3Iw48+imIY4ZXPPQKVTBXIZpDk1yE3cjLSJI8gJKDCuH0JH/rcd7BzugFaKKYTo6UAr7rk6Wi2qIFZmTVqH687NzdrQVmlguFh+m8LvJjSTExMaAE3bNigTKJSKTvfYj6RWkCgghbhN7/5DdasWYMjDj9cWsznec+n78RVf30csi7Fmp6dxbZt2+S7+d7jjz3GNkFAN1DGzp3bsXdqHpkkUrBLa8QgkYIfWbFC1oqWwjIASxt/PfV5bK6eg77RMdTm5pANs9rU3EzNVgsbN2xQlL5z507s2bsX+UJZcU2xVEa+kMehhx6K+lJVlmmxOodyOY8iQSKmtKHhE8wQCsUC6JK56bKZrCxBbamBbbv2YGJmEVGUYGZuHg/smsPjuxgQZtGJmR01iTzh5ecfipMPX60MJqHGv/T1f5MqCGDixwgzAM44+TgcfdTh+NOf7kMUmy9dvWY1JidnMTG1B1f+xVEYqt2PTjNC/3FPQWbkFAQMurjL0EBUn8XVn/oZlhqUfILNa4bx/HNP1s3uZ6eVH0vWWkjmt6NjY2g06hgfn8CePXtw+umnC/EbHRntWgYfnevtYYg/3vZH7Nu3D+vXr8eJJ5wgMyNrkBIPyCKJIgnxlj/8QUIblhkfxNFHHWnoYpxICLV6DVMzM6gtLEqo2VxOm4jBICP7NavXoFwpy6r4lOy+Jx7AVP4OtKt1HDN4EVavXG2pXauFdquFSl+ffvaYAnEOC+kYzWcl8Fp1Ud/n52cQZlJUaJ06bX3G4OAACnlmL4w5LPenJSDwMzk9h30T01hqJVhcrGF8cgq3P7wLaVBEGrcw2D+ING6inM/gvFPWY/3YANI4EpoXvPi1b0gVfSaxfEIuCHDB08/C6NAQaswj832YmJzA1MQEVq1cqZ3M6PySsw7HxuqvcfBp5wLZPLKrTgXKa5nEIY2X8MjjM/j4N25Gp5PijKNW45xTjrHgURmmhyzNT/svRvaz83PSKm4ELiDTNAaAK0dHLUVzUK5/D9Gr399yCwYG++X3DtuyRWkU79NchWUY//7vP0EUd1Cv1zDYP4CnPOUpyiYoeCKJDPwWFxcU+XNDcSP4qJt4ALV21SoKNZR18HDw4vwCwlIOeRCCphu2TdeOLYAsl/oUv/B9yjSE5Pn9bz8060tKjaNmA5kcIe+m5FEp5DA6MqwUVprPjZjNal0InO0dn8DiUh3bd41jZmZOIE0rTvDYIw+jkxIW5/qmmJlbxBuveC5WDPUjAP1vB8FLXnsl41kkxMi5C9MYFzz9yRjs68PIyoPw3e//BzZs2IhDN29CjYjS3Bymp/ZhamoGpx67BRcdsYS+0RGkURbZkTUIhtfL58edFn5ww0+wYwY49YQTsfagtUhSQqghgh7s3YMjFBQfqMHswqVhtADUFP5+zSoPmdqiefDE49U/+tEP8OxnPxv5XFYC88ieoYIJvvWtb6HWaMjMjgwN41nPehYKhZwEz6zANhtNo48tLLjsBYxmZmdRKpYk+IWFeW20pVYN/YVBBGmbS4rQSbUZtXXtSrlProvXYXyTybEWYICPNF/+nJrM7AIIMwSRAqFrvH4hl0Olr4yQbq3TkQvqRJHwiUa7hXY7xsTMLDpxCjrq3Xt2Y+v2HXh8zzxajRAnHbcF//mHu3DVZWdhzdgIQOyAgn/xq/86ZSrD3cE8cmSwgjNOPVFARTabx969M7jngYfR11/BYYceqhvs6yvj8ccex/S+Pdi0biVe+pQKiuWKHqCZFtC3+kiAaU4c4QvfugWnn36StJU5pfd/HrmSBXA4O39eqFZdsGXQKYMvoW8Cd3LL5qHnJ+HXjJwd2KN0zL2Wf7vpppvw2GOPKTikmTzuuOOwZcsW9Pf3KY1lbYGL3GzWXexBvD/X3aCG1IUuj7eoPopalm5mrEbA/6TRLjefXZiXxq8YGtFmaneIT1hsYM/sN1WAbIbWKVQAawheiDyBtEIO5WIBhUoRGVqiqI09u3ejVmtYLYM+P8xgYWlJiCQ3RL3Zxt7xSXzz5/diurpEDBdRJ8FVzz0MGzYejBzRUwr+Ra96dUp/YVqS4JgjDsWmQw6SqcvnCgizBfz+1rtRb9RQUjCyCZVyUbs+G7SRaczj2KE9GB4cRJhnKpZFFORRXrEJIQpYbLewb5GbyBbS4NP9v3o1a3xy0upVSYKxsTEtpNA9p+W9xRvTGHst/feTzzijK4ReTb355pu18ShcCpzvocaMrliJhx95GIcddqhuiJAufa3/UnlC92z+la7QinCEf1vaXNS6YqHgAB3TYH72vfc/jF07d+Jp55wrX01s3XCJ5Y3iP4eCp0JRcQw5zCAfpig6wRcrRYT5HJJ2C1sffxyZXEHK4HEAru327dsFz/J384s1XPtPN6Da7iCKAuTTCK89fz0OPWIL8gqeawhe/TdvTGlOozhCmMQ46fijEMcRWq7QsXbtwSoQ0Fc1G3Xcc89d2gAEYsaGB3F05hEUC8BA/wDy5SKCXB5BNod6M8Dw6AYEuT5MN/Nox3l0gixCpEKOzF57HIi733zgdR/5uNIyBmMffc81KBWLLnWCgJCudXDYAS/zuc9dj5e//Ar5P7+JPOwqH9qkSWzJT1NYvHeLzjN44RWvxre+8gUhY9RMvzFlkVTBo3ZyMwQy3VbetZ/9a7278huR36uNJv54+20487TT9Fr/5QtNvJ6hkgmymUSCzGWySv0YzdNjlfM5rXWhUkCmkEentqQUOFfIo9mIUHHPkMmwfgCMj09qA9JFvulD30A7YqU0QSbo4BXnrMfhmw9W4Kilv/B5z025GOvWrlVAcfDa1ejvryh9mp2bRZxE6BCISc2sEKTsL1eUfo0M9ePQ1h0Y6K8oTy6UiwhzRJtyCIoVtNopBobXIghLePvHb8DehTb+8tLn4vgjN5omOcxbwhKgkeA1b/8AOiHTwgD/dPWVCAPnHhJfj/eVQds8fMhf//o/8bznXaJrMrWzwoyle94ieKEIPnUC5ee+7K+vxJev/2cBLMTK9xOig1It9bCSrxe2TwO9Zel1XYK4EeC+B+7HkVu2KENYtnQs1tiuN+g3RiFv0XpWpjsE91kuG0jwMvXlAggQRPUlaXa1XsPw0KiCPX6x8ENwaXpmBq1mW3HYWz78TTRbHcRRG/l8gsvPXodNB6/D8KALkJ/z/EvTgcE+HLppA4rFAlaODQk0YJCkuncUK9qtLi65Wm+iXDKfy2NkcAibc7sxEFRRYP7JSleGwVUWGZZTcwV00gwKfSMIikO4/LrvoFGrIwlYnkww2NePjetW44Lzn4Yth6zDJ6//Mh7dPQ7kCtoI1175SgyVgLjREkKnyJZAKgkU4H1VMbhiGPNzCxjq7/szF+Kj+t4/eEFp6VPgjf/w//Cpj7wfiCPVnVi4sYoagSl7J7+FQQatqOW0ny9nqhjYexwxQ9kRU9ogRKsd4Ikd2+Q2ezV++V6MEEIrUypmtFnzJEi4cnM+E5hlLRaQKxPCjtGq1bFt+3ZkCzlQy5tNuqYsgjCLUqmCMJNDNpfFtq3b8I4PfQHVdgYED1fkU1xw8lqs33AQBomM8tkvu+Kl6dp1q7FuzRoMDvQpcFMli/wOmjWmBQxsmg3ML8wrNWm1Y5nKfBhg3Wg/VlbvRLaYRblS0aLxBmju+RC5Yh+QZJAvD2O82Ye//8x/oBU1EGYI+ph5lwYSnQpyAjYCFm8yKY5auwrFTIJmdQnPe9bTtdkCvjYT4t0f+xz27NmNv7jwAlx0wTnIWu7lavWe1cPCiVUAewUuoVNoCPG17/8HfnrLHei0G8jEEforZRxzxGY8/aln47CN683KxTHe+9FP4pqr3uSw9VAFIC6gIfIGTfOzmOb9/k/34f7Hd+D8M5+EjesZpyxXLL3lYebCzUXLUSnnpGw5MpPCjKGY2UD5e4WxVoUwbQeNpSoeeuRhlPv6FHizFkJLiyCHThRjaHgEYdYRWDJZdBAik3Z0j1a0S5D4MvGr/+av0vUHr8f61atlvivlfJd+ZP7NLsSImNt7sbqoaJVwJMuEQ5UK1jbuRCYXWuUqzzwzQMjiX5hBm/VUokhBHmvWH4of/G4r/uO27dpYbW4qMEJuW82fhZT+QcGwjNL5+7hZQ9xuId9ewrVvfS1ymQI+/vkv4eFd4+4+aWEiHLpuFd706ivQV3CEiwTohFZmpZCotywtKyf2QSECXPPxz2PP1Jxpdmo0MRIzGGN0WE7lrbCQggBf/uS7tUlrrOk7nMCTKch5EXMoCfHCt7xL5eIrX/YSrBstY3Z6BgN9BdUuKIRGo4Xdu8exa/dOvPB5F2KgXEahyHWzjIHxbzEXopjPolzIIlcqIUg6aDWXcN999yNXLiIT5pB1sVcmVxGoVF2qyn1QcbmpGezJUjIY9eCZMznB31z1uvToo47C6NCIBJ/PmW/0VS2PmXMn+jIq38uSIdOf1cEsGrvuwPCKYb2n1N8H1qLDIMekFDFyKBT7URwYQTbH2AG47ut/xI5FFnEIJpgtJZbA6DTPYM5CeTFWmAlk00Rwbzlp4bCDBvGH+7eDdLFcPsccVItJGJiVqDBu4Z1vfT0OWTmCX9z8R9x88+3YO79g1y8W0CYvkFS0NEGGcUsh362tJ6nxANBuyVfyXgnEEOPnfeTiOlqdWEAUOQkK1LKM6Gm1DIXMs9LJIkyWVTWWsyNRusJOAykrZtT0hG4kRSZMcP27r8Lw0ADyBa45sX76+ACFLE19TqhbtmAaPzW5TzB2QjdQLIPgVS5bRCZrha35+TndA91th7uMMQq5BdmsXJLnMcgCXv3Ov01POP4E9A/0qUzpmSI+L2XgoAjZ8ceIGQ8OjSDMpajNTCC751YsTe+WyeEN5ooFpAysuG2zBWRyZWRyJYT5MoqlfoRhFnGYw1VfuAW1CLpBCo4mnOaOJsyDebwHkidZQ0ijlrFhWGpkvuwCIZp9sktYcTKwhiRP4u+GS/B31A5FzTkSOwzdEsMna+VfQruMri11C7nGiNp1wdc0xdyE/EyRJDr2OX4RubAiXDhCYTZfVArMjED3w43SInBl+TtfqwJP3AFD5X++5rUYGBg03oDz8Uzr8rkMSrksysUssvmsyBSsMywsVeWCc7miaFf86L6hYQWM5CNQu8WFSN3n0fX2pNDdNPcfP/Cu9Oijj0bfQAVFLnpgCJonUdCP6I3coSI65rBipB/ZzhxytX2IOouo7duL6clxjK0cQ4YFCNa9aSZzXARWxXISfC5fRqFAn5TBTKeED33vbrFd6Q2I8qt2DeKelrrJF4fmn5NO0y28ESy4g1ms4AMGcYo0dsGW6E0mSNYJjD3kijq5vOruZAGrPiC+Gz8nNMzesWnQiUU8YZbD12nzOOSMfpkBmQiNciEeRXS8O2U+WQQutYxliex++NncuAS2WDEMgwSf+ofXYHhkRByCbM7cFO+3kM9K8KWC/Z4b7oEHHkA7jkX+LJcHuDgqjBl7LUB1adEwEJZkewTfi5P4+w2++rXr01WrV4vlwaqV1ziCFdqhpOrStBGhCjMkD2HjaFu8vGa9jrjdRNysYs9jD2JguB8ZmuACNZ10JQYreaRBCWE2L7+XLw0gn+tDjDZ+c/du/OC+mvBjZlOMSOlDpXUUvMyhOSWaRgrn0IP6sXXfEpKQ6R+lZygYo3wKRCogjXRsU2k8HTWZKYzWtR+M/0ZPyOditcuBWKxokc2ijeBJoEnarfi1Wg0XD9iG7AaOzl0pLuKzhgy+YrRbNbMQ3Ci0KjT9LuAM0wiffsdfYWCgT4hhzmt8wOAui3whlLknqBS12rjznrtQHuzH4OCQTDyYriZAo93R91p9SXEXuX9MSRhBJQ5V7Kad+n2A4Mc/+U5KQCOXz4hkwN3vH0j+nTCj427HaQfFxm5k2nPYsPEQRMSK63VE7Rr2Pf4QKgMVJEEWBW5ZMkizOSAoSvgQm4QBSQkD/YMIM+TlRPjkz7Zh20wTqk7QVwZMVag1zu+H1CQgK9Od4NzjNuC3D+xyTGBHLdZdG3tIbF2nkWTL2LMAMS1DYAJmakaBRdwkjCXSZZKmuAmuTE36uEyzYyZRGXRtugrHCtbN9RSaqIXc+Lwjlpup8ZaimZknN5/aLvgaMT76lpeif8BKtdzkSlkp+FwW+XwokkcumxEWQB4e01fB3glzfqDFmCXOY3qpij2zc5iYmRNPj7WCyZlFTE3PaN2EzjLnT0l3zyC48Vc/Tum3izkLSLxv5wsZFPDqeQoOQH3mUQwkS4iSNhb2PobDjzsJcZpFVF/Avom9QGkE+8IxzHcsKm52OjK7LIIwJ+bNczGYEkqzyRlfrKoQwyCKpVLyyK3yFWL16tWCbVetWiWK0Y7tE2i3UmTDMgiRkGxA16SFdSVaU2fXTOCid5pDWS9uD2/JaBIpdPpD+VwK1Qo6PjXzDFlqqzYV1yS0ErIIoO493WvyNY73T+toG8SII8IFGE+0m+b34wh92Rj/+IbLMDRQUVWQ68/r5sIApTwFTnOfU7DXaNZw74MPYcXQCmT7BjDZifGr/7odv/j5r7CwuKh7bjZaiq083Zv3q/RQjSP2DFIoupxb/vDrlB9AOpQ3W3yDSrREk/IFFLIhGgsz6M83sDQzjrSzhKWp3WB4Mrn6RDyydwaTM7NYmJ4WLNpqkDHCsqpl1wGjJUdOZIzAxgOqCYMaMlomJicRODIGF4qfS0TO4EvL9WnGy+VB9I0MYGx0NTYefgRWrdmARx7eiUZEDJ3mXi0SXcFzc7HkaigZwRZWDU1oKrSoGhd3N4AyBLo2x67hhvELpss6gEaBo29scBU2a6rgpjMLqTuReTerwcIIf8fYQTy4pIOV/UW84xUXm+ALRgRlbJPNBMrj89kcClTGDNCoV/HYvgmMHH0qrv+3b+Kmn/wUzaUakpibqS16FtNgGnLdpweedE1bG/8l2Pu2229OuSuIEgmWJFWnY61D9LnFfBHtZhXlPJDEVTSJ4i1MYms8jDu27sbM9CTI0m3WG8rzSXpQaZJa6FKIgCkSF5sgBzlkDeuCUTqmbhLyAai9xgX3xAziBTSBSptUuOH9RdIkslsYMwyvXIGD1q3H0aeciU6SwfT0IoKYKZsBJGCwaF5N2YMv+lBI0liCMNRALprzvd02JII0PW1cerFr6uBr+JV4eM9bFwnb/KhF/wbskC9HgXdY/ubnJh0cubYff/OXF6GvUjIGsKvO0UUJwMmhtTQAACAASURBVMnS7zM/A+qDa/GjO+/Ad7/4RSxOT6M6tyRhE71jzKB7UZxhULDhLz2Bp3sOX/0L/njbzSkrcTmmR2J0UvAdVYoYZbcaTRy0ZhSt9hLSxhyqrQQ/fGQntj7+BHbu2KViDh8iH2bRYTWo1VavF4kN9CX+i5pLIERmNKILMHap98Eyxu5GuVA+q+DfvQYyWOli4u5B+HTtVhv5QgnDB43h8GOPw4bNR2PX3mmkCWlGXATD9wn3d3NZ19JkqRU1uCPfq9cR/OFiOizBP4OYSq5nwN+HzwR8XYBK7zeUrbxzEdlQkCvXlqkc1+ysI1fiZRefp3o7LS7jWaGdxEyyxO/p5/OYHjgIn//eDbjlxz9WQN1qNlBfaqJea1hmwazF1ROM9r1MF19Wc2cRfX3k97felAouDPkhbDeyBgfGZwsLCzh43TraAbSjOqr1Or53z0N47MGHsG96EvW5qpkR+lpqRxoKsFhYnFckOjRozYsKimxFtC1ljrgBGEGLlNhCqVDosm60GZyvtZ1sixfzvU6jFMn3PCT3GO89E2aRKRVxzMkn4fjTnopHH92joE60aaVUbocpTTOzTpaQNmTbCBPmmy1OULDnzCbvn7IkV4GsIAV+jlhpG8HKjbpfFzjK1MsCpOqGMaoXsYEEr3j2GTjz6E2oVAhG5RWRM0dnUpvPBsrfp4fX4Gs//BF+8Z1v63lb1RqYWSxVG0g6ZlloKUzY5t+9lRKwxKyFn66mFXNxMvW33/m7VACNfEtGwdxAqYJGbQnDI/2Wr6YdAS3fvO123HHbXZidmUCtWrWOGknGkSmcxs7PzWgB+ojiuQVQlbOnGdIvKv9OCJMwr1AnSlDWzW7UUDHv5ykkBkl6TMtZXb+sqMxOQ/3DFQf7cNqZT8bw6i0Yn6wJE0ji5cWhn+X1fDCXOFPPq1PjPa/fkD7g4tMOw3Aphxt++wCa7Eejm0jNaoWsx9HfuoYNWgLhDS4IzKYBWu2aijtJRFcX4W1XXIzD1q1EX39ZcY1RpcgoNnpVe916fOM3v8F3P/tZ1BaqhgoyaK7VQeNET8brdxtCVX1ZFrA2rCd8sMdOWY6hecG2HQ+nytPNXuDxJ57A0YcfoXowIUxT1A4e2LMLN/z2Fuza+oTo0Z1WJLSNC5QLrSDDYExtU0xX2EjhCjVSBEGvy3mPj4yJhjEIpPb5WrUE3omF5JnGEZQx7bTXE41yLdRsfHAVLW/GTUUNDczm81ixcgVOOvNszNbLruHTbyrfsGnBIz/TbzSfx1twB1TyKT74mmcp335g6y58/IbfWZSeWPA0UExx9tGbMTg0ALJvdkzXcPeje9FJXJFILeANtJsNVQJzYYLrXvd8rBoZRH9f2bh0LgilArI28rXHHsO3P3s9gnobs9UF631okyzJFJNt07auXmFo0cTjd7QuAW8eCEnNTbJ2IcewbeuDMn584F27t+PILWSjLGtbSsJDp4Mv/e5W3PmnP2FpsYrFuVlpL1E9+TYX6PhArN1q6Ca5YqwZq0ecrcmwuEFsWxclCxGLY3HLuNhWwrTAiF/LdW+XirkHUBqnaot1wfhWKh9t+9hAGiQwpIC1h23E5iPOxkw1Ul4fKge21IqWjXi/zGVkm4zBqQI0JHjds0/BiUdsEMBF3ttbPvNTcQUOO2gIVz7/PAz0FY1k4hDHWr2O93zlF3hk15Q2ra4dR4rASW8uFXO47lUXqWuGtHFDLRkQk4oVYm5sNf7hfe/B1ONPoF5toLG4hEg0MWtKZdm6G++4YpoXfJeswt/njJwiM2+9WsaDePSRe9K5+XmsX7MGCCx/FnTioMqApcMgwAd+8GPsfvwJzM3MoN2oi03q4dzeHnANFiCCRi3nYjKQ4W5nBymBA0er9bvS/5uoIXljZMowyzDs3ARP7fZt5f6BfdVQ+DbNGbn0Dnvw1/RWhdaHPpQo0Nia1TjhjAswOWtAjG16mnWn9Ywj4tRtVFcoCgNc9+Iz0NdP1GxYz/APn/gOLnv2Kdi4akiVSNKoSZfig6saFkW48iNfxu6ZljYPg150Wog7LP7EKJWL+H8vvxCrVq2Uj1ddnSRMRuO5DH40OYWvffjDyKUhlhZrmJ+ZU3Acta0TNqZ/d5aOz6D18B7Qde/qn+x/cJCzBG/BAIId2+53Pt7Ff0w7HFNUQUkSoBp38I7PfwFRvan8ul23smTiWpx1QZcoehCIQmfpVakSc2kGLs6HEV4VE0abzOWdaqNqSPs8iMRqYLPe7sKdPupXHaDXnCk1dJvK5azd6N3FCXzkTDY0GHRwAOdc9Jd4YjvhYm4qq6AJ+KHQ9R/dHwXPew9w7UvPRH9lQIUUami7k8itsXTKz+qrlJV6Gb0a4iy88rp/xXStZe1EHSvwsGWZ3/vKeVz3hhdibGRIVVG5L7c+gysPwT/dehN+8JnP6P6qMwtoLbHjJ2PDHshWcmml4hkH0BizyBWaHALLTKZbZHOMJHEHd+14kFVHV6PmbjI/4YVPwd83PYWPff5fZY7n5+ZkchTYREZGoKaxYCKBqJKX0YL5luGUwxKSjh7MdhzfZ2M7WEnTZ6n6xc+3yNkHcHFkkasEaVmquXBXePGbRDEhNcBPvnCsV6/9phXcIHI4GFq1CqefdwG2b20gn83gnGMPkRn/7n/dxZKhLayvwgXAu192FsrFigRPIVHgCgLZxMh6OmOOuC0XwveOT8/gTf/8E3EXhAa2WNjpICVyl3YwUAxx7etfqALNgOfOuecc2nQMPvbv38RP/vXLlAZm9hHgksd1LsjRz3rmAsiUZ4ysaWtlcDV9vA98icR2K5+7dz6QygcIraLf7MV4yBMP8YddO3D9176h/LK2uIimIw9GrUj1cC6l0DUKm4tSKNrCEaZkBCn/Sf5XR68hN73XHHOz1KqkdrnUR8iYE7KCq9AKHMs7Qu/3voubVQ/sQRS3v2je/UQMml5x113vO987vGoYz3nui5GPs3jSYSsxumIIP7nlQfz89ifkl3NphNEVfQg6EV777FPEFciRaCJuQkEAlPAOdSDF6sSp1uoWOacpds/U8Jnv/Qbjc0TW2GjSRqfFGT8RBgvAu15Hwa/A0EC/TcfgtqcVXHsoXnf1mzG5fatKzlN7JtHh3IGOwcm+zNoVLhXJTwhxZFDx7DXQwp7ZK7JiCf6egtcOcRUkXwZ1ayfB/+qhB/HV730fGbJLG03l96VyWRE/YUMPanAgAS9M02XRsHWMdtqRmjFs8gQrgMbn4xdNF+MC+kDW232TJFXarsF766mC9RAlfflYZt5tPrZNd+MIEhBcOsWF55qqGOKsAu3Ohk3r8fn3XgeNYBChsw0aeQFMCjzbyDgcgDV1wxCdFWIwB7aBM8hNMTXJoQVVDV/Khnm0GzU8MVnFxFwTESNql3qxBFUuhDjs4DH10omHILIlkC2vwOLAClzygov07/pCFZ1mB20Ol2p7opdLZl1G42XmgzplG07wHAph7CbPHbQAO9i9/T4J3hcTlArqhYa6Maj/z4fux5e/+31ZBX6xyCL+eQx1frL/2uBJE1CxaItLTp5cAtOwTgdlNxjIm+dljSWJoGpUoR6Dw3TQz74hgdP8mQV9rO759mb/wIpJnCWggBmWW3rJoIj0Lr4vRSFfthjFggYce8KR+Ke3/r3VFBw6YN9tuJBCHocRMCAkoqaRCMp1m/pMVtHsy+BpFmvkXlzM0VvA6xZKHIrm75vSKY1swV21GVz5ssvlPmenpsCCe6tJi2kVSJE/3CaSiXdarfV0d2FO2PrzFN84S2DE0RDBrm33plbNMTOrFwtbtxunlm+dmsK7r79eo7zYfz49Pa0LksMWkbNOPyZcm5W1SIKXRlOQbvAAr1UgEcL5TW9R+JnUdGo+f2Z0T7fAtmUjL/ohRRYjdWnTLK0q1bL7VZroNibzYFW6OP6M07ESG8ZEU88qPI2z0kg+tWvHPvPME/G+173WWQubKME14OcRMeyicc6dMDKXSVfjlJl2GzbkNjvDFlcA8trWGzQ7jnVXG7VJMgWs2nQyfrvrYVzzt29WlD89OUX+F9qiSpu785u7m7Y5KrndiOvqcZiAXusKNZIZ14qbYPsTfzJT74TufYU3lwRdluIYV33sY9izaw9WjKyQORNAE2bEvo3qNk7MI2Z5ES4ziv797zTPxhcvyHdj2ZIkxowVaRrNpjB3sk206TizjTmcQ798dcsTNdQz59I3+XE/G8fh1EqpOJPGaYcWSUkE0zZHRhC1i6VMoNzfhysuex4uOpkNJS6ecOsiDXVAUrfjV1mLzQEy6Hg59LTgys3qcTvcv6Z7bTapOqSQm0XBbHkEJ552IX744O342LXv0maan5xGu2Fz+biBvUWWn3cWdVmbrTZgf7PmjO5XYAJn3CNTv/WxO/aL5gwNNRaMNgHBlzCDN33ww9ixcyf6Kn1inwqQcflqa8nmyfmgg2wer/FKP8IQfUxZAvpO02JW/riYziIKtrWCg2kaF0OQqcMCLE0xbdKmFI3bNpt2tcP0lwNEe61gaPc3EiK50RgzeOugZgfahlwGI6uGcd0rL8eqsgE3VoFzNWz304EIoyeKShP3Z2Toc+lQ7AeLDZQ1+c3gt0vQUUo2sPpobDzyqfjmrb/CZz/0QY1dmZ+YRrvZURWOFsBruy7hNJ2/M/KKZWTmEi2GkrZrjay+z79L45949Pb9BO/RnS7+y3AmCXHVJz+FHTt2mUA5k6bRQKlYUdNhxFzbTYOU5udC5IJQ06fYj81FZMrDpkBGwuz0ILmQr1XFS926ie1q23eiIkuPxKaxFE/+TNQsg2xlrknRJj6uoYVu0uMBdCNR8Xt64nxFjUGnf5+lPMARJxyGa156ETLUSEfA6DXRvaQLm79nFT1vgnutp35nXG5Xo3d7wAWtXY/sovK1R12MFasPwse/+Gn88IeMqYD5ySkkkbVs+U3vYyMGsvwitd1vCG/apRgug/EKwPsVY5iA138neAV33RZhUpECXPu5f8EjW7dK4H0D/TKRHkWrL9ZMu5wPCYwnpfStVMx3aT/lkk2x5AJzwyzn2AGWFmwciEG1ROIsImcngP8d8XTjsftq1HKRpGsJnDb5a+vhGR73jEZl4YJfrTpHlbQVRKnuEDeRLZbxgueci+c96ThZGwWBPdMovUXxwv4/v7Ms263ULTd2UOhe8N4qHHfmy9AulvDcv3yumjKrC1UsTs+ps9lrhH8uWVjH2OFoWD+mrbsONPU9FrHL//f4x4GC38+H6Kksgvz6D3+AX91+J/ZNTmPlihER9Kkt1NzZqTkJQ0T+lEOEbKJUg+PHOEdOXaaWRlhbVluRsebcudIqW6v4ZRUxC9i8pgkAcUQNPxOPVoAFE2M1G2BB089Ie7nO76ZfMo5wjFsjaFre6ytwvjpHAbA0zf759771FRjmbDqW5vTN3tNl3hxQl/ea7u/Zm3OBNu4f9gzuOiqp0nbbv/m8p5zzKuyLY1x8yYVI2x3DTJbaypq8Jve6VFpemfWsZVPe11NxVJ4mXOuCX+HzPRhG8PgjtxnE63DcA4M7H93f/8QT+MfPfRb7xqeENDHlZb5OwU5PzMgf2pgOju0IdeP0nTRRjNR9p6lpl6dsW+uxiBcy81bb94vnYwbTKm/q2aded6NOjTxiqZkPZJbnxskMujSG16LwhEp2HL5AUEn4dyR3w0IKcfNGp4VDDzsc1778Ik0IEYfAWQxtHIcNeJN7oHk3VpFx7Lw2+2zGx1tiHYnla7uCKdZJT389djTn8ILnPxedelvZUmOxDgJlPiXrjb+84PkZJlRvqYmeWvpLOSnO6Y5pdXHC/yR4v2M9hZQ6e8Xbr8bknnGR+VeMjarkyKDFplVbfkkiBunCNKNcNM1+4ZQot9i8GU8j5mf48aX8O6vaxBMOFLwewOHntPISpjRcW9YshWRqpeVljTfT6tunVWdz2YgXGrEDVhKXLUyKKG4jzGVw8bPOxAufdCJsAJ4Fe70MnD8TuIJIY+76Qpeyu57ah4tcZOks4+GfmXEkOOWcV2M8buOSSy9Wl+zE7n2qzJHZpC9qdU8rOF2WBW6ub8CGDysG8jELKdi9BTFqvnoi/2/Buy2QBnjde9+L6YlJ1BttteV2Qkb35JSRTsVBBqOYn19AqZRHu97UBAcxWVUAsRiAi0Vs3LTBEEMztQQnyJV3wEi3b8+CPbJNJHAVAARDIAxp1m3OjUYnyGotR/8+4PK+jhrPh+a24ZeqZq6+73237iVuS9Yjq0bxrle+EKP9JBwaC8i7pgNNe9ctuUaGLqPVW9NurOAYPb0ECsZHYQnHn3s5HlgYx2svv1xDlnZyXm2DzRd+MzlAxltnx67pFmnYs+i4CrbZrWdgOZay6p/WsVfwvQHRssZ7wQPXXP85PPjQw4hbxqAt9pUM3NCM+hhjK1eiVquqVZjATnNpSa1V9SUifSZ07ThXRyf6Z40PXviU3XIwxfuhpis3pbhcNUlpXcrJkHy9VarYR+bUwpENliNtmVJqhhtQLCF6mJobxY0oMbCIrNsYaSZALk1wxMlH4e2XPBMJ81ovfJ/f76fJPtbowQDE0LGClFHUjPcvSmRP+sshxtlwJU4454XYWp3Ei1/0fAl+z9YdaNVZOXRkDnLundnWWtBqGBnfSCeCqx3IJUw+g5C9DS7rkOvz6R0F37sjvL/v9a/ezPzyjtvxuS9/w7LTJEFf/6BAEuaM1Wodo2yhyqZi3HYaTTSX6IsLaDc5A4+948s0oS7o4Lhv9PMH+kx7Tw/BkprB4TBuSoVnk0p7e3y8sUwcO8VtBy2My2098GHgi6F/QtkI7XYJl4mme3AcyWUXnY3zTtwiq+ILJb1BXG+6p2v2cvV6wDF/T5aWmpn3eX2mshknPekCPLQ4gZc+7xIRR/bt2IW0nWoEqwJAFyAIqnYceW0gujONRjGkUabd+3xNyzAOo0y8h+T/O8FrZ/QM9vc3vGtiGld/7GNokM+dJOgfHNIN5Esl1JaaSvM42WpmchqDlT40qkuW57rOFAqeXz618IQLQp0+mjeTq080Abvac7cq5SY+9lokWROhaMZt90CP37wezu1uZpfOMeL2kbpZF2sX0+9oxrKhZr2vPmQjPvjaS01QnAbta/zO5HqLpXtydGsfzPXGAQdaUWsGseccXXcqNh5+Kn6382G84YorpNn7du1G2OHQZXYYWVTuhejxerOgoWb6UuNVYXCC1wAoR34xsGx5uNKf5fFeyH8meAVQKV7+9negsdRUF2uhVHInOXCEZoyBgSHBrgnZpBwQmMliaX5hGRNwJUW2QcvvyiVTUNY9Y4vEvWScd+1mZ+L9QtJskg7uLbsXJr/3gjzK9Z2Aeydg9UKdGhQgrGB5uD81nuwWfn6x5Kp7UQcnnnQs3vr8pyFhAEuouMubN+vXjd499O2kvHzfznKpIdQFgT7RC2Ks3fxUrDvkWPzbHf+J9//91UJMJ/ZMIMP5/4504S1ibwbmTbfGonhwxroQDFdx5p9TM2RlnaX5M8F7s3Wg4FVxSoFXvfNd6h1nixRBbqZz9DPs1SItScWWZlssXVbXmrVal51DhZF2OJ/LefDC792pE/74Ea6Zh0u94HtNqyyGI17sf2iApYP+iw0XfA4fsXdNsouC2XBh4IqnYBlvgMEqNy3rBmq7Zg09l8ObLr8Epx++1t7j8IflWMG1TrvY04J5l8FrQ7syc7cBw0f+/FuMw4+/GANjB+Mbt9yIT77rOmVDCzML6gTWejm+nA9Yl92FabH66RwobHgJXSLHprtBEY65a4qSLAd3+5khsTmWmyGW/5bic1//Fm659143FaMtrlkmzxw5oxnsNJXkp7MnnKldwBMZ2k2n4baQojVp5y0f9GP9ZHxI16Xrkbb/5lAkE6blrUyXvNb3+lrNv3flym6q5iZlmbl0ubnKrsuRtoKv0NURHKDE/J7CXrlyJT781iuQURVwmW/vJ2n6dTrQvNt9LWMBFoAsX4P0miNPuRylgWF89LtfxLev/4Lq8NXZqsUVztR3i1yyGm5su+M19Lo1tZ7J3xPSJtBlkT3nBHD+kCJ+H9X3Ct7vpt6gjxuVulptpXjLe9+thgIb/l9ANh9qxh13HevgnAUbtRqqH7Ma3G6Qg+5GjKo/3Z3M4HYhP88iV5q1XuybUzCXaWD+HjXT1VGfeMxIt1DjxqHZ/RsB06dy0pSeYr9lGGZ+fQrpFZQuzUWH1nDBOCWw4connHo8rnnxhSb2nqi+F9b97/L7XsFrI/QIngcRHfekVyLfN4D3f+Oz+P6XvoL6YhW1+bqUwbtf8fnUEk7XbVmO/8+ex9rSLO21vn/OxPGvMSjc4RqPPfzH/blWzkQtw3+2BqoMyc8neOW170Lc7KDW4I0lqPT1axIGT4KgeV+YnUfSbttkKJ2SEGkBPZZPky7SBf/ncHdNvhaH3wSvmXZuSrSgzq4sXErYZdosQ578DAIcytVpDTgqNJsTx603S/Edtt2mDBdc+nEhSiFdKZYLau3ONpuWNunNf/UiPO24TeikjAF8N+z+Gu03wn4Rv13VxTLELXyXTQfHnv1aZEtFvPOTH8BPv3ODMqOleTaX2nxc+3IVU5uNLlqV/u4yCV+UUXOGS/2ISfrfi1vAYhrP1fnfBN/VMHd+mvdb//CJT2DP1JR8PRejUCxr5CajevLp9uzcI+5Kq9HQOTcqtDgN87uXBRdj4jpSINMxtmARPOkhG0gj3YSpZY1f5ot30yEH3XrBy5wTruQGcaNWbJHoIhxh07mTLnjj0tRumCDNdBOtuufoNTE4Oop/uuYNqGTMTRyYvvln7NX85Y3gy7Q9pj6NcNLT/kYW6lNf+wL+5bOfQaNWQ7tu8/a94AlWeRTS8jKL6Ak7+9TWc+q8sBOljL5knopnL9i8V/B+d/aakO5iO43nv+fabbzlPe/TpEvWszmtqTzQJ23rHxjA3p27kXYiDdRv1xvIaEdyopnV5mlNBJa4yF34ucCpZbMuLXcVbvu558uf+uBOiuLDWqmV48eJ6pjfZ27PQoUGASjiNW2zcwNcW3NPV6tcjidhmC7p9dZfZ1VCC/5iHH/8Ubju5RcjzbigqtsHv0xqOdDk27+XBU/6uTZJ3MbJ578RnUwGV13zd7j5t7/B4gzZzHbGzeWXno+DRytYu3Ytthx+sjSf+AnHovArk7cDDLiOkZo3OqJ38/iS6mIVu3btxPjUtNZgdMWIxrsHjz5065+ZehmVnsHCvaaeP9Mkv+Kad0h41PhOJ0D/8KBQqpGRFRjfvU+CZ3GmVeOZZ4ZW+QYGCp5+U8CJS1XsnDTDnHvNI9l/vRG9F7/OaaPA09jGnrkqneBLsW6tVu+jenseG0fSi5z5wMtyca/BDvVzgRWbQvjF2IQ+ts5zdAb68YaXXIInH7vR4fcuqncuwt9nr8n/7wTvLdqJ571eJK7LX/ty7N69ExM7d+tcnA/+w1+jsTSuruX+8iBOOvlctOheOA3bATtqi3R1CmIZhgoukzbM+jlfryyXnTQHCt5H0YEt3oEab4fsxPi7D38M+2bm1KPNHJzjVGTys1nMzM6onMlyIjWe5XCBIq4Y4mqpsgJ21lsGhaLNZ9UZKgfUwL22q+/cgSbGqzNwg0ebLAekPZOhHWDRfWgXqBhGYOe8+SKP105P+jBugINhXVRurdNWziV5k6dPXn/t6zRShfN57b7deXvupn1N35t/g2z5xSPI3FSNNMAZF1yJJhJc8BcXolpbxPzEFJ739NNw7ilHKzvZu3cv2u0ETzvvL2y0W4YFsZY1RSqEtuYILU8P/iHShYO4FfASgeD3/03w+2m94FPpu4KSG/90L7763e+KK+fPNB0cGsYS83Z+eMeIGA1W55x5p6n3QZa5E+ukocayuyTmQAP23HVbq5fNpu+y8ILndcjtY0DpgzSZbwEX1o/HyFb5rzv7zaXConJzg7ISyE3D9/cya/wm8FG+ByIMjLHNEDV5wEEbp55wNN7xmud13ZQ/dsz34nvBd69Jp6TYhtVIA384NvbsZ70ZDXRw3nOfqfR3bnwSV73kAjVu0Idzrs2WLUfisCNONndDy8Jj3kQbk7S1bgKyZLKZvtHF+U3hu3pdJuAF3+vfe4M6X8mSeXQRqRinaYqXvfOdVp1rW55bKQ8Y9ZcTSjkgoVnXMIBC1qL9ZsOgXp9XMxU08gT71SC3wQKy9c7v3z3bTWV08C6DthBhjhg1I1gKuqPhTdQ4agg/Y+P6Q/T7J3bv0nc+QYFM4E4kgKRUKVvzB+/XUbcs6nbDC103Tm8qJmBJPspGnw8OD+Dav30lDls5pJGsjPIP9O0y94Ejk9AySPDGG6DP56HHZz3z9SCP6annPRWduIVocQEvOf9EFDJZNHiKRpzg0r94EZJMCXc99ATufPBe3PfEds0XaqlBdRlml3vTBDHWsK313GIcp/H8+ZEH/7AfEaPrTx2I0xW88416KLczrv70P2Pv7nHU1QiRiK9e4kmPBGg4cG9xHs1qTa1XFHK9VlVaVGBHiqNQ+SmWjI2I+ok73jMU2PPIfV+ZzFo2QKWYRV9fCUdsWounPOVMnHXqUZpLx5YvBWX8X8+YEl7zZzffieu//WNN6uJCsAlSvt2Z5WV83R5wWfPN9xuubwJM3TGqTBU3btmCj7z5cimdhhj3VO+6m8ALvksv94pEjU9x1oWvx2IS4YKLL8D87BQKnQinbFyFUilEK83h4aklVJsctJxBJ43sEAWlecQ+HATuXZvj01tKu4xzCDQLHHT7yAMH5PE96JaChG7o5wbEdcsnwHd++TP85Le/F1onDh1CTa6iH6HpnJ2e0lwZGh+mEJx/y9/zNTTBbe1U46bSzDdaNVWjSOvK02wHGR1Pyu5RNimefczBuOaNL0auWEa22G8bZL9wX2Fo128vM1qXq3V8psvecDWaHfo6etrlnOrLdQAAIABJREFUUyVoxs0aeaH7s++6oY6GBSt9SvxxqHRRCS574bPwgrNP0LHf+wvebWSX71NYxuJxfYc8H69TwbnPfAlum9qFv3rBJToAapAzfJMY2VUrdVgz14vsZimmKw9zvT1NWemby90Va4Dzh/O2Pjxjhz/buA7boA/ff+v+ZdmeAwB6BW94ke0C3TiAxyfGcd2nPt2tvtHskHdXLvcp6FuqLii4o49XvskTpjsWCFr0buNLKBa6DPo6FWs6ETauGcKpRx+FVZkW+ioZTcV68gXnoNTXr5mwYaGvSy1aFsufC94s2DK/3FLDBB/90vdxy+13q7ikESqOmOhNvQWLPqOwdNQqeNZBq0O1dW073rRvbAj/es2bNQv4QMHrda4L2QteZVKXiTQ6/XjqBZdhW20ef/mi56BVb2LLyjE8OrFP1TVyA3RapROumLLi6RlY1T1hROtMZI4HkCyPPekOqGQzhevuleC1XC5a9qdGdjnc3VV1gu+ZlUYm2LWf/5waLSi4Rt3OSunvH5QF0OTLZktNlS7YVGBF/63+OlKtoibWjo1gKBfgyU86Fcds2YSoVdcD7dqxC7XxvTa8MJvBEccfiU2bNyIln8zNxe2mTeLjOwxeW9ohjTpE0U2B8IvvovrPff9G/Ow3v9dG8C7OZgAZ1cprfm/MY0pj7dR+8BCZxwxKTzzpaFz7+svUb2iwrxVgzD0ai4auwCqCdm6u4vvsKpz5lOdgMm7iac94Cvt8sFSr2rkBpYIILzygkCCZGkRczq5Yh/UIxT3ugV3NPpfJWYDrqWou9uJhN9qu/5PgvU9d1qYe8KHH/33qhhtw59332KSodltBUqWfB+GWMD0xhYQDfHnkB4mYmVCb45gth+JVL70Mmw9ejdt+eyNKGaAl2lVq57W1Wf1b0oOPrBhFpZDF/Ow8CuUsTjnhKE3PDDlwWX2qjnPnTpdga7NFuAFml+rYPTGDJ3btwa6du/H4jr1a/MgJNYMQe+d4+JHx69XoofEtHk9YVohebIGLHDUtoGUBhCAWZVmq5PHuv/1rbDhoTFC1xQn+9Gsz+ewgVgbhLAp/Vxk7AkcfdxYerc7geZdchAyVqNUSNsIDhIsDA8gXy1izdr1AnJGVI1ixYrR7uBKHJmkABYmjUUcnWEQ80pTdSY4E09DcnQABEUhO5/CC7+5q59QP6JZ2Zn65YGBPFePGu+7B17//fXWnkBUqfD6bU8co/dLsvgkcdtBKXPv2v0eZGscFcQ2PRPTuuPVmhARIskTAlufMeoKCtKbTckeXt3Dc8UcjIjBT6dO8WBFn2XHSbOBHN96E2+5/RFOz5xc4vIEjWW0fdNpskDDNZuuxPUkWHNPKgMdAneWDE4Q0us1ghxQ57pqbasXOVf7dmK02pqUV1TE0PICvvu9q66qVK3DBoOPiJW76tbFmLfXadPRTMbZ6C+6c3o1XvPRFiBZr0vCxdWtw/AnH45o3vQOtbAGLSRNtXoeHKDLOIOdQQE5TgheLiC4kxz5CK+ho1Bt7DgXKaWqwgu//UfDLhYHl+vay1V8G++ZadXz4X76IfRMz6g8XQ4XDQfI20+bT11yDdSvYnWrvtvzdH/CT4t67b0UhZKQKneaktIqATj4vTIAFHg76L+RCVPpL2LD5YLTSAm689R48uGsvanEbDRI7NayYAmCDpAmEEueu9314nnZERJGLwaEMPJ2Kx4ISG9XwX1f77hZ12AnLmX3uqBYej8b3b39sG2rzi7bAAa/VUimUtfvXvfQv8Mwnn2LxkGsIUUbAymPkOABdMmmKE858Psr9Y3ikMY0rXnwZpsbHsXHzFnzn+i9isDyAxRCYojYrM2B3bIp21EQh5LFsAZpRE40kknvlBGveY7vdtJZwztbNZTVFVKd1c6Q6Q46H7vvDfsGdL10uI077C16+xEnRV6T/8StfxgMPPGoYfKOpAf2CU8MQ737Da3DcxoN79oyVZ81iJLj/3tt12jE5Y9wbGvTnqE9qiswVcffObdg6OYcmkS4e40VtijqIOHyJ6ZXNf3CsXetatSKFaWmxwDHqqYQnxorr+KG14EZbaiyKPqaqHUu+hbyOXtFcHfbQpQl02CCPAUkTneTU3z+EQqmgMXC8xvzUAh668x489tBD6Bvsx1fe93eu/85Gu+hxCbeIim7m3yqgIU4+66XIlSq4c3o7XvXyy9FXqOCmG36CTjaDe2tTmFiYwkJ1CUnU1LNVin06P2igUtZz54KcKQAPbK5VUa0t6dACYhWe/MKAUCdq8339Ayb4/YKXIOmJWLVnl928+6k3g+IDfOTrX8KOfVNYYhM/o/OGjfwuVUpIW21886PvWw4endYbVSrFI/ffaV2jYYDhwiCWwggP7d6N+3ftA6e9WD5uQ5DIfy+VCAtnNJmKJj5fsgHLImW6IUd8vU6iEiOVymzRr6ZDaDqIjUenQDz/j/dLS6Hed3fsyMLCnH6m1WAA55s0+R4e1yZ2TmQmv6/cZ0WifF6t2SPFPE47chPWFAjqOJaP8n8P2bq9n6Z40jlXIFcawKONaVx26aX49fd+gioifPeeW7Bv9x4020ZWpZvUHB1X32DbOT9P5wNx+geha83+56idpmYOCH3V8CgrK9OtqavIC753Vy6nKlbrPfBrP1oRgEen9uKr3/sBduzYY5F1DC1UpVREI47w7fdfi4JGoi9/+c979IE/ycT+6qGHMKHZM/TpHbFMleY5/0QjQ65dsdBnlOwMO3nKBssqYjWfyvr7gU0P2YxtDsKzur6iXYNzaX2kyc70coPZWbBkFBV0BIv8uwNFOFmDMDXblnTEaLVuWLhmJLlBDBqz2gKZBfTJlXweh60exbFrVqLAw/6kOZbOMoA97vRLMTK2FvfM7MSHrrsO1/3j+/GlX/0YtWZDKHwjsvI3mU1SRTe7lm3q/L2OSHcDE2z2OQcgG3pJ39/f168z6Q2Asna2ZcH7kqXPT33x/8+jvP1KpMKtA+CaT38Ke3btpeHRTbTqdRtRlglx1MEH4QNXXWlND1phnuGQw9bJCXzlxp+iqeF/Hevf1rFlxqnTgmesLas6vyDghydcqFhCwZfLNoudqKF65G2gAdeVAmabcRe75sGDPNpEwjZrQ76g+eHlXj3l+SFkJvmz74ilC+Ln8h54f7wWByl3hxvFdlIlf6fqFzLa/DwpQlF8QgIErVAWmw8aw6lrV2GIz1EM0LfqRJxw8tn4rx33497f3or8oavQzmawZ99eo7g166jyUEhWNDXg0CZue1STsuY9ERX1ZW9aAI6Cp1vSc/oBlAzAKfyuqfeIneOieTLhfrNJnML65gCvv2EnxTv/9bOYX1jA7CzPRcloECJbq3gWXV9fP77y3ncgdLXoWpDBh7/2VdQ4NiUb6oiQYp6dtBS0+T0yham97FtX0NbuoJ9DgrKmvS3Oi1NbtO1gTXB2x4F6mhf9Hx9SftpNxTTiAidulG0sunwfq3vmq42Ry7P1LD6Ym511J1waLz+roo65EgqFFoAADg/3NdNvk78ZTXOEO6d1G1hlYA/LKszzmYszRz9qzTqcccTxeMa5z8Efdj+EY9cdii/9/scKPHfuG5eb4eeIE9COxGWk4EV2FW3dOo/ov2klaUH4HDq/p5BDP1FOziEin4BuK3KnZfYKXubCC77Ht/cGdDJSPTVzL/x//+1NuPnuO7F376QO/SHPnmANtY+jxZ9x+ql4yYXn4+a778FP7r5LTY8WgNnid32tZ+BqegPPb8/qYfg1Nz+HFStW6Pw5G49mw5asvNvRYpG5qwEA7nwZ1eXdDHrz3bQgoYY38ShuGzHuJli6oNAPHKBPlabHHeXMS9Vqd3gSNwCFwvIsn4MFG97nAlubq1U7FoSVNzfixRNMbWRMoHHnNKp8xv7KIC48/VyklTwuOP0sfPOOG/HE9m1CKcW2nZ1HvVF3/YghWi2jsrE3kW5LVDNOJGvUVSuxCdaWnjZ9+uh6+voqA0a+3E/wPbTh/yuo289fU1vCEFd/4iNYWKhpGjUVkBOyeAulgQEcvPFgXHjaSfjp7XeI8EfByyfnKNiiLkchtohLZ0JVzTS/3REofSbAYI+WwOY4WRrlhwaYZtu5NLxml11K4Wv+KwVIjbWAVZ29jrTou2jNh7puWneqhI/CuxbB8d1keplpMDPgKRsayWra1p3ooTMAjEfohyiYh7comxuBFUaCUayzX/6Cv8SetIaZ+TnxG7Zu3ar8XE0scYLq3LxNv2KwFxEws1OuRGyRGyNPYXkursrD6mewdjVuECrGsuD/jDpki9OFcntKH12hH3CI3ds/+0k0GhGmpucVPTZqNtRIc2Q3HaJhwjR/vDGdZknBMmcv8EhR81MUCjXMTmCsKHCisBgQSUhu5IiaHbN8COIFLX2n2aW7oK/lG1ivl58OQplgnbjhzJ4f70n3wSDJV+Z4v0pFdUJH3tqomVE4lyKAhNTuXM4CLlLIXYaijdeBzDADRDJ2+Dn8PSNsfbabK8DTJ7wbsvGwsY5Uo5AGDlqJJ537FGzfuk2pGcvNtCzjeyeQNFpoVGvabETl+Kw8a0mhk07T4vApy9U968jGwtrBg1AtweXxCmj8cVVdyrCDGLuTMRzdYZmdIF/TuzE+8fWvYNvEBKrVprB7Tmmy82dC9K8YxvCYnaXOPFrRdKXs8GRrCOC1Cjx1SVagoKofTaHamkJju1aKRQmRm4BmmMGUmgl0Ph5HtFD4oSJdHlIoQTnrQAvgF0QWhgER74dkkBxHtFkwyCyDGtls8v1sTc7oc9hDoPo5aeWlopWRHW9QAx8IALmxo1xs/seBDxQar6l5QI48yvunm2H0L1eSy8taaAN0Yqw6ZB2m5+ew9uB1WGpaUBrX21iam0dSb2tsvHx+HOu93IA2JdQsmT/3zub4s0GEOAnn+TuuwYP3/j61xTlghu2BPt6pucesZQ16ulb473sefwxf/vH31DI9OTGHQr6o1Ee48+AAVh98sB1Nmg3VDcoGDGq0zLNj4vB1FDoXRvmyNCpAlnVoQqSOOSvf6o48UWzSPQrMDiCgNjJgZDWQfycSSC1TuYSU8EpFAxa0UI4M4vv7/WYmMEQLQjfB82vM1Gd1xKgd48n4wE6I4t8NCzALofiGpedm0xpINIPVrAFfTyvjLSqxczWNJrZxma61kxiHHnOEaF08XbJEhm0mr3N2o0ZLhwtatZAwuKdpG+1a13Xt0lZwshGwJjNXabz/7t9Zde4AjfcVq16N9ibeC/9AwXOo39s+8SE0mxEWF8m1ywp21TSMXBajBx2E0dFRTM1OyXxT+NTu4eFhV+hIBXuWSzbtsdJX0QBFLThLkO7kDC8gj35ZfMB0y7c5G8uFAxm8hov5oxOiLGswHpoFexFTsB5yKV/L+6vWaoKhFQsw/qDbopVgOhVzWBOjbaNPSQDq+TOmLgtWtAIUsqhSOm/Oavn6HV2PQxap8Uz1CELxWjOTU+gbHtIZczT9tbkFJM0I84uLQv40ccMxj72LcmLt1hv8rF/rVvIbgefsulnB9931X5pzR43vFayn/nZ/2fPDMqazHAf4zfC2f/4Y6jXOrKPW0RTxBApCjQkqgwMYW7VSJowaNzDQj3KlpIhVJyGHduKjR/WGhgal+eaKLKf2zQKeI0cky1MmqWl2HLdZCk260vwkoiuWHtq1fHRv8YGVNN0UrU6Mpbrl8JoL70AeDwFzc/HavE9/eII0iqddOl9NzNxo2NY7wOfz2D/vheZd13Puocv3Szgh0/n+OMYSz5yhu8uRjt5Gp2F8Bs3+cz32XHc9k6/xusppnLBAQ9DGjZ3pys8Njrr3Tzd3Bd+bpv1fgveVp672uw/+xNe/im3je9FuJViYZ4pT1BgzPiyPHx0ZW4EWz1UNM+Kr0ReroNOJugQNLqhP88zk53XiIjeLD4i48GZuE12b16FGWquz5eMKLFmo0Gxao3Ornq2UyooXFA4hT9LH5LPJSyfzRXPeeVaeTZ82KNfq3/LVDgWTmddxIxaUskjDz5J7IP2cfATm7AUSSjtyORQmT6xmcEaloPnX3D926XJjRG1Zvdm5eRFccwULUvkZjG98u7lMfc9Erl4l9WCZZh264FOm3R2lEtx3501/jsk6qEGvO+Dsdf27p8nwwL/fct+f8L1f/grNRlvCTHQSFGfR1+RnVq5eheHhEdGFS5Ui+ocGFeRRmymkpXpdUCwBlmqVg48NauTf+BrCrjqpmUOVNJ3aOPq95t80gEMMbCqXMSoM6vRQrVqdecx52w4r5rU85GuZQYQGMXIaAyJ7boQqwR9r6ba5fPzZ+2w+o9c+Rur8PWuVokS56ZtKK4k3MHhsNPRMrD5SOAzWuGGZxtWjJtrVpgpdeY0zIx7h5v8fkE15gft2NNERPMXKtZmL2+i+ZAn+J8FbU9//LvgDTQzR3XaY4m0f/QjaLaZACRYXaoJZmWpRUwZHhvXf+Pi4dn+pr4SRlWMStARcLGjB+DN/x8XwttyEb5G3bwsiBs28lILSyVGJ+V47KcOdwuQHIzmki8+loNH7Sofbe3/pDyrQcARC0pEBONwYLHeaqY9ccOioVu6wQglQgRpLp20dHMQgtMh6gMiFlvdzTDsF7wEm4QFRpBm+5CJG1RrWj41hvLooZJM8em5A9e/tJ0TDOnRWgM4vW+4eNsKHa6QgZtAF51IE997xn1aW9RvCHxLYE+Xv5+cFCu2/KbzPd7w+XP1PHxNyR3Ig/X3o2oxo+mmSy30VbQI+RK6YR2WoH6NjY1Ys6aKCnIJdslTLmUlh9K7rlg/P3zP9k5+LLWgSvu9MGzWLx6eyscOKIkaNtrZmi/7FPA1tdoyCMoEthuVz09Gy8JHVu8+TJxrN5dxex4rbgctadDcPT2NgOQeIm4NTudsRSoWi3BTNuoE+BiX7moHO8AlYX8igWmvg3GOOx9bHHkGLlb/hUUxWF9BkZuHaprgpmSlYCuomePAZVX20MSuaKJY4i6nYwUrYstJe8N1u1P9D8JYO7F+qPbCO8++33Iwbf3eLmB6cwVpvttRMuUTggSzb4WFpACtffYMDyBazGBoelpA0BsydskBSJk210jidHr188iMbH0mioKnnmTpK2RxWrTyWgosiuQsiiL5TlwvF8WFWvDEXwE0gi9ED7XKz80RMjVmlptPXu0FNis79MaQy5cu8dS2uAB/bZEL15hYUh2iKSKGoZ6LF8CdcEtvn9TIF+vkYm9eMYSxbxrZdu6U8737b2/CO970fLUcKFQGTpedSHpe/+FLsG9+nieIkYDTbCRaqDdQ7MaqLiwbwaPCT9fzbKBEneEvnTK99D1ovAbFX4/k6f0Cu9+8HCp6HF73tIx9EQ1BigrbTiqjVUV5PXj2FTAtAXln/cJ+IGMLdXQ+4hv0zHaLQchbNKzjiyRAO4aMrkOnvOe+eu52WhP6W9Wqhda58aahcRr/XEaU8Lk3om1kw/T3DyZvU5Mjyap2k6Q4Tcpi+LI8zb0a/srly1GZtnhangwxi5042ctiMAB99cxPpYAaetunm5pn1KiCfy+Ctf/VaHH/EGlz7/z6I6blFNYf84js34PmXX4HxxUWlnzwHgHLaeMgqvPkNV1j/gPy6I7XyKIG2O0/HWciY6SspaHrUAMG9t/0qVSDUtfUuRXP+vSfH685e9b7/QMH7rIAb4+d/+D1+cvNvEUWphh00G0SnClocbjyadZqrQl8RpQFjklCQtBIM3vh3wrvM8ZmG+d8pv9cJGHbwMXc19yyHJnJDETvQfdCMavKGQZTyvZq358azuZRMGAPsaFW6CnXwdlujWfHj2H07811CdHiBdx3i2jEbaJpm0XJUFxbtaBN37h7TNm4QnW1HbN5lE9xkwgYyWYxWivjsR9+PsFNHOw7wzre/B03Xa/jlz3waL3nNlWh3mE1YZsHPf8HzzsUZZ5ze03NvG2B54ANPgmSvH/sarC5BjZflvOePFLztIPtyw/APTODdMZm9Qtfe2a/pwjj3PId23/g4PvGd7+pExHbckuAzjvLL06ZKRUP1hsaGke8rOnDFJmPzxpka0ZTTRZDRQj/JtI9HinNx5+dnBaHq9GWNPOF4VAI9OSFryvmzLO8yFfIgi82zITQqGNMFYvRc3ADcVLQAOvzXCZpuh75eR5u61Mn/TTUBx6admZ7pNjsYNsSAyyJ6uQimkJrQGQu4oiWjpVLzZbkfV5x/Fs6++BkIkizGJ/bhwx/6FBqMUfJ5vPTi5+Az//YdTdu01JDQc4APf+BqHd7EjmGnx12peSU0hWZgZ6VkUdoJtd/1+/9Ig2yha+o9r/5Auavo3zPHpTeN86aef6/Xq7pxfsjMUgOf/eEPVEsnlEmTT1x5lpMeuLitNjYduQUxazOu24MPRvNMn7V61SqlQdZTl2JgcEAIILVJp11ns1Z3dnwyXkSMWB5w3NVuRvochpix4z1d5G8Rrx18SOaFnbbp/L3O77RN7eff2IGExmSlv6fAVZRhwFZj14vx5ClwKYeCNxZebB4A/y03ALqrorQ8aEXIxsDo8BCe/8wzcfYzztPnXv+5L+G+ex9WF8xJxx+HxflF3PfYE66WwbMA2FxBwb9dNQwDgNxhB85S+yhMrogNopyOqfpEwXoO7rzphympyl00rqeTpjdt6BX8gZvCd4dw0hU1MQjtSBKal0/827cwtchTlFM0eVhRjuYt0YwXYs4Do0PYfMzhOqyI5lY+OZNRNWtsbMxKmSREzMyocEJzPjQ4iGLZXIUQOmnB/1fXm4DXfVbnvmtrS1vS1jxbnk0SOwOQwKEUuKec9gKnvbSXnsDtgdIUCJlnZ3A8xU7ixHYcGw+Z54lACCWkgRAgKVOB3lKmACEOGZx4HiRrnqWtfZ/fu761pdLnKk8e29LW3v////u+NbzrXe9C7stROh91Op7akJ1nLyRufEK/EykURSYVaURXnpFb8TTVo3zNmmCxEzAD7Ispl0zrrC7bkr0UvW7a0UK+IDgmsIbrYx481cLJoVHNigXIaW1stL/7vz5g7/3QX+geb7h+kx3vHlDf28qrr7aHHnzU3jx8xOlgVVXeJVyWsS2bV880Y85C7sTO+aPxa6E9MB0Azn+88LViZUN9iRY1G7HTwiew4D9tgj9e+cK0jYwO2ugINelxEf1cLqzCKusb7Ma77rGRsYIvvAK4aeuht34YgGTalp5xmoIh0Z1SHqqyLHRgTnN5ue19Y4+iZ1JBkDayALILXACBovrsRSzk9PrJ5k/eh0UQ2WIKfzzuQzAEAVeImSq/m8gbs0UXtVlIocYnrKWp2V7ZvVufB/jC6zWpuTTOnM3lAZUC1ERGrhD6Q3iXtYs/+yn78/f/iZ1z3lU2ylBirFxFhc1ra7G//av/0973Fx/Q765ccYMNDY1YRVW53XfHbXbeZVfa0PC4VWRJbSutOldtJ5+yxD591pkl9ywnrTx9RrHbvzczrox/w2FUeZuFr6irNQTw3E/8UZVuloz4fzH/kgKdtqGhfhvo7xHPjxMERCqQhViiaLbveJ89/Mx3bISceBoR43IbGhq1wd4BASInnn6KbxLkT5P6BOkPp5vFZNwZlGA4dt7hWnDWa6qzK3VT/bxCD9JFk7xQwmvUyiWSoSNaIHikaSq2AMeGzm7i2zvxwjti8bGHDx6SLw5M3a2fa8fOPumeGkZ5jFSuYOUVVXbRP37CPvahP7OxiTErL5bbhZessr7hwVJ9YF5Ls33yzI/a6e97l+bW3rr5DkG5bXPabOXyK+zK1dfZ1DT0NLIbh68/9ekzbemyJQmjjyFFDmyJZJkImRGTKRZTvJEKPL/8wVPFLHZfKdLMFzcwG579r7Ges1X7+o7bYH+fHkplzjFx57MnHRp2fzZjX//Bv9mLr79pY1PTIhYAWHQf6xad6MTTTlYO63VkR76Ae0XWmPaBQSwmChQUPKj4IaoEDWtyKs1uhWyQkCtRq9Vc4eVZOPgEU4Jkqd2X/LMDO0Q+QtuS/JlX2aZtoLfX5+6Me8SuOCBlDWqc1Ewel0VNp0YPlrEs+N6Vl11s/8cZp2mEKcdb6Np0mV142TXWOzis3ye1nN/eah//xF/bO05/p3372y/Yt771gjbF5ZddKM7ffQ89rnurylVZZXpOGzauKrVuz14b71FMGH6pVO3Bu+TZo9bw6399ugi6U54oxrFDSsWXPwJrwnxwUnqPd1tvbxf9jG7yknBh7K5Ib8SRs6Ld9rVvWtfggE1OeH38eNdxGx0ascVLT7BslUt0ccpFhkgsGnrU5CpFnypo2iVpFyYPd1JV7SPNggZFCkX0r0pdRc5pT4gsTnoBRpG5pmI6HKsKmrphnLbE7/Ue7ylV8XwGruvc6jDHeLGEoP2xKW1rqLV7d+2Q8jUz4tHpY2hh7A0sziWXr7KB4RFt3urKSmtvbbKPf/yjtuzUU2zTplutu3tAz2DjxnX2nef+xb79wve9M9bKpAmAZbxhw7ViA8emi8XWus2ur6TFn12QUVT/mx8/W8RsVtbVKZUKzvz/38ILiJiatKPHDtrxrmMOqGRhq4xbQ0OdR76iKGdUYXLyAtQp2LRlduODjwsRm6bXbmJK7wG/bu7bFjijNlPmkxdzHs0L8k1Yusw2hY8xoN5Kfb+6psZPU6RsjAdPzRK4GRZN8irqn/NNhO93yNZzfRDCgwcPeaahnzlHLZqrQwtIFbIUs0mnz/XX5RLmtLfZI7t2WFkmFW2o7lERTGij3KgqekW7YvkK6x+gszhj+YpKa21ttE984n/Zyacus3XrblR9o6q6zG7eeKNtu/V2e/XNvUpr2bCtrc1WXpGxdetXKo2L9Yrhi1E/iawrFrw0MQPYmcD3Nz95tshfsvnqmVGUs4oAsxUewhocPLDXBgd7rRZeO4CLUgLUJp3gr6JBSnV4qAzrpazJDp/IVtj6ux+08XEXIOrp6rburi72bhpGAAAgAElEQVQ75R2nWi5fJVpWTIuWdEcmK5WpoBITsU6NjothorKsumYq1FnDahJjSAOHiD0hhsQhWqRUL1eRZXLCTl12sv3+dy/p+zBo8dke3KWWyoT5RwnWT1XS403ZwalvW2wb1q6yGvAHZt8orYJXMCZ9v/8SBxeKduXVq6y/f0TpcS6btY62Vvvfn/yELT5hia1be4Ng7o//Px+z//7f/9SuX7fZDnV1C/cA76+rr7X/9t9Ot7/+m//pZUNflFKNI1SqWWjJzKT0TsLb9CUmjoIWXpEqIkJqNPgjiYlQdhbiNWl73nzd8hUAAVM6QbW1TIScLFXUWCzMLQ8eU6uHKdpUQWaNhzc2VbRVdz8iXzvQP2DDA4MKZIBvS0UWsPKJcUX2oH20PQnmRA8Gf54ia95P/w5lZvXDe4Qr3ZuE2omQmS3X3Ly+48fVri3oGWsSfjHQykRsEOkyNWzoz1Te5Tc+eebH7NOf+JiVic8fEqN+qpW3o10z2F9iNpWCQCvaimuusy4NcCK9q7B58+fY587+jO154y372teeUoFn545bRL9esXK9DQyOKACtq6nS2Jfzzj/b5syZ4zUTLdfMBogTrhOffhLiNbGh9TMWXgUH8B3pw/6RyH+KfNlBv3/pRWtpbVSwg4hIZUWVFgUkiTcLnhxBhEqjqp5VauFFa05pVKE4YdduvNsK9XWS7oSQSLfI0tNOSRRh5qP5o4oqXq7CdXNQfFQzQUrB4kaD9IirCN9NLd+LKR5TkB3wRZzgNKqssgmdBsq0iaemVm91nrjlkD0rFq2hps5uXLfWTjnxBCtOjNjE6JBNF9OoD6EiaeEpKKmBdEjmPsy8HnwmY2vW3mgHDxyVqa+qyFnHnFY755yz7Stf+arteeNNETm33rpBa3HJZVfbRKGo3L+utloLf926Vcm3J1WwpK9TMu+zOIhR7ZRf5z+58wzI3bNF/Bw0qap8zQwpD3CCFl8gycKk/fxnP7Y6nW5Mablm0kRtOJgutAHzoNVpGukDTQnw4NOAez3MwqRduXqrldXUWqEmp46b0aFRW3jCPB/Gm6pPXjIlGnWFKZogRGAYGxcaqNl3IVGCWeUI0cQwNq7UjxPeP9Dv7ohWbIE1nutrkzKIIE3OUPqTpETGoSinqdMANR9835/amiuvtPKi2ah634gbmLfjA5SC2RMBltDHXKWNDg1IRzdcJDgF6eimzV+wPa/vLZWYO+e027nnnmO7du6yvoERe9/732Wf+ew/2NDAiF199RoJOWBl6eVrbKy19etWWyEdDA9WnV41m41DZ66upyQL7ylfVCW18DwsdGkrq/PqWg2TwALRqPevP3zB5s1p18PioSslKjI9sqYEYPBv0LMQHyZ6la4MHHSkRRPY4cWNgl25ZqsNDY7ZZFJT/qu//JDt3vOGjQGkZKkbx8hxCi4geUNC0UT2EE3Z+XlAoZxexpqqmRLqUlKB4JRE+TR2vrc3BZ07DQtOOS9WT8BMgXbirJ115sftr//yz60yBAJxIakEy3Pxh+sNlVrcVOjigQPYTIwjYDaDi0RN5LZd99qvf/Vb/QYWcV7nHDv/gvNs88bNNjw2affct0uiDj/50U/t4UeeUNBLCkxgh4u9Yf0am549blWAES4v9QSIfTNLVj3a2tN8HFkGsHr+AnyKOSwkCQlFvoUJ+97zz9mC+XNLrUPUkTkdBG38Hg/K25jSlIbkU928uYq0s2UyOoFu7op2+bWbbHQUwWL3ids3X2vNjY32Vtcxu/OpbynIms4SKnncgUw65n1oYKjkNnhw1No5wQgmkwpiobzWjXIkMLzntJ4ZzPhgXTPbSySGgk1PeD0cw/+h95xhl1580cwpUtk+gTZJf4aYQSdM/p0W7TQYSBOoIVKaDfb3ei1cQaHzCCnFPvTQl+0nP/2Zfrc6l7M5nW32sb/9qN1//6M2VZi0u+7eqef58EOP249/8gvLVVWoXeqEE5fYqacttb/6q494FlOqqDocoRi7VF53/19q2UoFptikmV/99FktfCg1lFUjLwKJYdx+8MIL9rYl80oX7sAIxREP1hzzpuqWFpRJjZU0BjjJMVIfZ8b61CQPmKbsipWbbWh4TH6Mn9+983qr1M8mbaJQbhseecSmilkrpJ1LkYeawMjQqDN3ktwqAaLy81SM8I5ZFzwQ8yY0bpPbIOAsFZhgoKZIHez702eeaZ/827+xbMYBHW3eWXNrg7vnTYre8oQLCVPuuZUTPMrLM5rS4dCtT5f2RSmzJ77ydXv+hR/q3/nKKmtorLWLLj7brr9hs7W3t9qKa5dbTU2t7dh+u/3htf0im1SUZWzBwnl24UXnys/roCVwYAY2jgifR12wF1980d71rneVXIBboqQfHAuPaNAogVoNufekff/57+gimhpqZ/htSXXaETAvd0bO7IvvBZAwO5xULyrgGjwAVTm0vNwuu+Ym0Ydj4W/ftlYkTtiuba2tiop3fPmf7EAv4gRaAu3eqfEp61HBxrn0sF2EUSeeuQKxSCeT4qNOoEy8/8y7TxBKKLdcJmNn/93H7S//x59bVZXz54Xvp8jeEb0Z90c2EbFCtGPF5lIRKfUE4ttHhocS3Suwe8fSv/P8D+3Jrz5dGsXe3tZqly0/Rw0mdO+wyeEu7Npxjx093qvnVYuSRUOtrb3u2pIiJsGoW9YY5SJH6qQP/kucwzj1EeknU/+sOmlYNAYHEUA9/fRTdvLJJ+qGCXLYcW6yEidb0bJDnDxQmbBZYzuFf6dxozHvPRZDQVW2wi5cfr0NDbvCJH7ujm3rhANUotGiuyGarrSf/eFl+9Lz38O5+jUUnWHTfeyYn6BUD4/F8YDQF1dky5ioHLku+IKZzW9pspvWrLD2+nrvLk26PCI6pA5dPcA0GCk2gOP4bvaDCqZzLDVtmh99mANZiluWJJU+i7j6rz/9ud13/yMKRCGcNNbX2YpVl1p1dXQQZ8VfuG7NRhseG9ZmbKqrs6rqClu95pq0FgCSKY1TQhGMx1my6SVqmd8Hr9GhpUnzVz/9pky92o6GR+0H33vBFi5aIOozJru+Nu+88SLFjBk834WC3SRi1nkgihjl99ko3sHhgVROKZiozsCvmaxdsXJTCthM379n140qENH/Hu9DuZQHN5HJ2LV33O8AROo2IVXr6+3zjtxEeIgALiJcFt55Zj6bDbPN6Xpww3orKxu3wnSZGD+FIqVTb2TgofC8iBf4S2QE/AnCCWLnnD6PH/izpImfNOZgzzJwwQcl+eKE/Dob9Pe799jNm7eKOs4haG5usFWrL1fU7uaYg2V21fLrQEv0LNubm62uIW9nn/0PrgyKi0nxS3AHFUeAxaSNHHN3JLUOd5/ANU3+yPzyJ98octqBQr/1jaftnW8/Tdx1ghcWlO+HooKCiRTQOfFgZgge9fN5nXOVdsUpd7NeUSJMRmcKC3Xt2lu18Fw8alcP3rlRHHTyScAKoU78fuqfw7Uc7h22TffdZ4VMJbwTmxgfs5HjA15jV+UpzVwTugbxg66TolVDy8rmbH5tld26eb3oymEVwjopABRVimmODkBxjqJZg00nV5WYupoNk1IltzJZUchp1BSSmBpK/1OKpdebdR/rtWvW3KgaAYgc+fkN66+xyrx3DWsDT2ftokuvVhNmLpe1zvZWe/s7ltlf/MWf6RoEa6eqYty74whpzFnqsIkMzWv0qbmCLODn//rPRdifzz33rC07cYnVVNFYjyKEY+Z6gCB7oi27VruQqfSQ9drU5kSlie+7frw//JK/LRSsurrGwZVCwVasuUUiAgA1oH93blsnwqWbZg+c5NNTuTWTqbCqykSxKmZscHTSrrt5i40VfIePFt0X47OrMlmbP7fT1lxxvvD3J/7pafvO935gnS0tduut14t4ETlt+HK5nOq8TjUBGqdYFLCkJOHjv5JJTaFxIHv6fHoBFAzGwMQU1AmrD1DMad0T41N24WUrFOzyzBoaau2mDSstW5Hg4qLZm2/ut1u27rKKcsx/xpYsmGvLr7rEMpmC1iWYxbMnRUe6GJM9ZMmTJaahItyhNuxPn3+8+N3vvmCnnbo0MTxc4iNStWC3KlKW6pQL7Qgpc/6+m0janBOYQt+7QI00CpTXw58bEUyK6obZVWtvsf6BARVramvydt8dN2vufHkGnRifkEzs4PPnvDrn4zNnePQrV9xcaoxQWiWt16w1NtZZ59x2u+DCz+l7Tz3zHXvyqW/a/JZ6u+ULG8UbCHMoM5w2gqJvYbyJmyC1rcSizbqbixgioiosgtqjmQ+LsGAqAPlrneipDt00akVoopXZ2ede5oTMigprqK22LRuvs0yFxyZsqPvvfcx+8eJLum9g3faOZlu9ZoW08pIivehlIe8+E8DGjJ/AFhJHIG3agLgzG1aeXWxrb5NClSSzcg5IBMghdAzfLUDGNdD53ynGng55O5J3YuLPKQQoDYLsQJ1elkOgsDdNTE/blas3W08veDX4ed7u2L5edfuKLPECVsSDLKjOcdpwG8C/nmZlbPW1G0Wj1olSX7gLLpRnM7bkhAX2+c//g0zwd773Y3v4sSdtYWujrb95re41uGhebk3zWCPVic2VzL3nhCYNHv6OSS8FkOL50biAOINvmBIXY1ZziJtc6U1bMVNuZ597qTpmWNimurxt3XKDwciLrGjjTVtt3yFK3rRHl6mCt/a6lYp5mPghYCqGKSWmUaSVgqFnz6FN4JIsgdZryjIP3bamKJECpj4nJQf0UllwuO1cMN9n8UhznNPuu4jXxIWGuY/GhdmuwLMGtxLezZq1q1Zvse6efvW7N9fX2q6dN8qiUL/WZ03RxeradVLByniaKECoSGlx1G6+eZf14S6IVBWJ5xQYMQh44aK59pnPfkp0rkNHj9rv//CGnXbyMlu0uFN0anrl8MVsJty2UjivcWrhnPvuZVUWLJfzThgBPtqYbr4DyOHa3D07WBVBb4xOdTTZlbimy8rt3PMut1GqotmsNdbl7datN6q8LZ6AmV276iYbHByWBauryduczla78qpLne8fbVJp4UMggusrtYZhOXhuCUAS6kmwGdnFU49uKfJwpJScfGz4AoEwqTpFJEmRI3xiFEViZ4m6m7a6pLaS6A+vj4fA+7LBeGRXrtxkXT39+vu8jlbbtPFa3xjlDiCRiaoZMgkjwWzJV6NQ6WkJVmPj5tutq+t4+r0Ka2ioFyO1sanOOjpa7JOfOlNmloCLY4I1IXLOZXMCmlLeWLIirpU341pYBLF1vX6XXh8m3Is30eEzG0SLDRB6dv4MQ8QYQnTWLrz4KhtJHT51+UrbsWOTwKuQTrl6xY02xgiVsqzV19baR/7nn9uHPvxBT1Ol7emB9ezgkc/l50o92ZRcO+4mYfmy1jFo6smHNxWJ3Gvzdd6tAsslpSu6UwV6iOL693kQ0XzAQkTBgw8jOnfzk1QhJj3FC2mxMEGUVq9dt8WOdPWqy2XJwg5bv+Yq158LkaCCYwFkCyx+c2tLqWMmINC77njE9uzZ50ui4MXZMvnqnL3thIX2d5/8XzpR6MjA2OEhEUVzeh2EcuuFC/NbTQydNILUv+dMW9+MiC0kD6vx5kkpOymGJ6hA7ztTxp0hiWCqBABZwS6/Yr1TyOAVVOZs584bS5ItLOoFF6+wTJlr9rQ21tt1668pSbUQJM1G61iTCLi5ZpWpIYKAaqaRrtRdWAusreKsrzy0qYhpAjiRZKeK9y4XonRMunBJICDVvLEQ6lWnUpceXpjxvr4+q63NJ/66CRCKFEUdKdPTlq+qtKvXbLajiCRZxk5/x1LbeMNqO9blFGJF3DKvvjC4ABSZS+yeJIT81a88a7/4+a89709SnpA9GmvzMvX/++99DjubmSAM8851VlfVyE3lESdOSKMTKWPIQFK5VueJ067ollUDBUp1Sh+9UMXChPXDlJcoVknXPho6FOJp6GLGJqen7LLL19nwiAsmsJluv32jmEK8fnh4zK5ZeaO6Xri+jpZmW37VBdbYWJ+yJdq93QLp2SSOXUi6qlsoiUXF4k9Oem2hIFZQ0TLPPLHTYf3EEC09iFS/hdzoJ9bLmhL2Gxv3CY4CRvyUicqcfocLUJBFPp6CDPHjk3+hpLnu5tusq3vArDhuH/nIB+3sf/h76bROTjnOz0KJbDmbNJneV71ykwX70Q//zb713A9SC5F5kakwaTVVNbZkcYedfe5ZJb8dUzV0ipl7kNqQfAqVjLPex/vrPHMQbSyJL+kBaayIl6rDWkARE7CUBhGT+noeP0Nr1sZELpyYARZxttwuv+I6G8CHp8aQ23deL3CKNHLfgWO2+dbbdVX8bltrk61bd40GNrAxSB1j7h4Qt0u4eWVR1PJZqXb4eFwkhJviNHqAE5b55y/vKEpdKqlO8QbSR2WokJoVsq7QkM+rqUDyImmjBEZNYKWO0tR2hAsI9E3pA/1psQkSiLFq3a12+FiflZcV7NzzPmMf/NM/MXYlpd1SO1OKntX/HsP1Un9aVWXefvbvv7SvPPmML1sCLthnNZV5W7yo3c694LM2gFxYdbV67Fx0AMq2F410f0HhKqlJO3PWeXze9qTYJQ0+ZuEduHLLhDXxTCe1Zycp2IgVPNjDiqYp2slDL79yvQJTMY4yGXv04S/YxCgzP8yefe5f7BvPfV/3xeZfvGiBnXvO3wvoYWGVVeF6RVObae2KjVLadLq+mfmBauWachmXzDNP7tJ9STSf+6P5AHpUak3izSXMM6szQ3LiibvNRXDS/cykScVRjEmSXlgETqmiYtKJyQnbcMtdduhIt0zW+uuusCXz5uk9AJMUF9Q4kBTyJ3yPVqXmlhaJKtRW5+3F37xsDz/6pCYS4YmVhmbM8tWVtnjRXDv/ws9pEfF3LDqxjNIwtRNFFO4+XlIkImqSK3ljI6cJV0Yc4q1UTufyeAewKXHVWeyyjDZXTY2TUBzV45ky9mw2G9aVsq66+gY7drxHz5Hq0UP3bnFpNdi1W3bZwf2HBSXn8zn7m49+2P7sgx/QhA8xmypcFSwieFqp9T4zd1WCk9lwMUJFC53EETL//JVdRS+0ZA3/jE9nN4cEiSDNFO0TaHHyWTy1IScqNLtesqOSFnXmZwnqTREP5ghUTOlexuy6m3bZocNdetB33r7ZMgValLPSveXhYvKxHIj3ElOw87kWsgvy6FxFue3dd8juuONhMVcjd6anLJ+vtPlz2+wfP/spvScPRi3XqeUZEMjTTp9Dq02dsIMo7tCdwzw4ZStpfrteA0aRhvTOLnzAk/PBQNTlgZvDgzoJNMxvIgnZqlUbNe81AuqH7tta6nK94sr1nl4WM1ZTW2nXrb7GqvMMJUjCy5p26WNbWUzkY4LVzLrwjAKMinm6cnFYsDQFK/PNf7pLZd3x0RHh7J0dc7SoAcWyMCxqgPwK4ngoY+jI5RxXTjVn2C+8nofKe0SKp0i7psb6epHppJW5zDZsucv27ieYm7Z7d22x0VHXguVzaY863tWtMnFbe6tj0gUX7yNvlpVJzYq3bnvEo/FS9cuspjpnC+Z22OfPPat0+jhJdOnILKv44+6BgI2TpDRITSGkfIg4OOvWT6+3OuHyAgQhaJVaRsbUYRvQKe8fVObIhlIQUar9Y1k23LTd9h44oh9hrR6+f5sXfjIZu+SS1Z6wZZBmr7atW9bLGmDXBBOnnr3gAgwMuhvz4pLrB0iBi6JNqilEql1iCX376/cWCWIYBshDr6eBsqxMZkunOBEWuUBSIXwtUOv8BfPVBaN8PeXamobADhwaKvlOHrgmH/NwKirE3CG6WnfzLtu3H8Jh0e697RYbGOwRT46NEf1uLmrkSo35KsfxNWAHiLSsTDoyW7c/Unp4oZbFaxfOa7eLLz1P2EOASogQuniiq2ViNuvqanXvwdlHWw8zEOLE9Oi3d3R446OkQV0xm9erkjcrBhD1WzJrnh56U8esQFFyJCCgGbvzrkft57/6rbue4rRx4r3nLmMXXrhSXAGRMatz9oVbb/BYIJl0hiV7FuLWhdgLy8VnKT7JmA3098t60mAZBaUA0aTg8fSXdxRJCWCv8tBZIE5+Hb3n2awWW8EWQgac9sqcbhqzjWaqWogSpTp2VcmspGmVIUYUYANuZMuO++2NvfsE2Ny49nKrqnJFDCL+uXPnWm9vt/h9mHuiUTBqmgoamMhUkbPjfT3Syt207eFSJOtgDx0nRevsbLeLL/mcyq0jzMqh0saJ1agSBBRzSblaOtNKrSR/htCR3FZE9TktOm3bbAoWU0JNqUGzVPhI9GtMKbUGzC/uM0rWOqmSP4XoMWZfeuIb9qOf/ruXbqen7aEHtrklmyjapcvXlizVkiVzbMVVl800iRDHJFfiwxbR05mWRWVD8qxiQ7ju3ozsCwuuRhA+876dq4twzcnvhoaGdcNNzc06ZWwAgistSNJiV2SMhPew5/IaQq+pkS4jovp1ivypPGGuBQer6lXU6afosGn73bb3wCGhads2rrL6hjrr7e21fGVOFqOmNq9AL4KRfB5LwAiQvC8SsmeZrF2/8Z6S7lygisQQcNXPOedT/6mowoNtaW627u4ebQQWX0UgJMxSB02oWChQUq48Q1dSeprN6p7AFbAexD3yqakti4VXL37aOPLvCXbmT8Ajspenn/kXe/bbz/v7F6bt/vu2CBc43jVoN2zc7nX5TMbOOutMe/97353qFR6QBtaRiEkJeaSJM5uGFVBPcJcY/IzI+wPFyzz12Db9fn9vr8y6JjAg3znOhMcaO9bVJRlSpQCa4JzznF18cadWCRiQP0Hsl8DLBXOl9ZYqfT7IB7/j+ey22x+w/QeOyjzt2LTWxidHxbEnIg+aFO+Zr8qnaNwnV/GAWbDJKd/dW3Y85sIJjhK577aiLVzQaeedd1YJU/fqmJ8WeAEekfsQhND04b5C3YprwISWxpmkBRQ5RYOKvFAliXBhDQm/T/AoboUrIThlc7Q2Nycl7kptjH/53r/Z40885fWfqWm7686bREP/2X/81h770lNpgTN2w/oV1tpSn4gkXq8I0Cj8tQLKcDnJCmhRU2XQM4yUgUiZI2OZB3etLerBpeCovb1dN0KgI5Rpako36qXHENrznBRhQt6UBSDCZcE1hVGRI6ifpxj45SjiuBLkuH35q8/Y7lf32vve/z778J+9x6oqMtZY16AuU8zf8PCAhuqRaYj1guhPmhwtl0JaODFht+583KN1wff+8Cn0zJvbYuee849Q9EvmNkgkWB+v4nl/XnXeCzDE6ywms2DYqPj56LSJdEnVskSAkB+PPJ6MRhp7KHcXrLbOhxPFEEDh/lOTcplcx+4/7LG77nncpssgik7bPbdvsInRcXvya9+2X/92t1c1c1m7bftNNlmYSDAwFctE7kzgTqCGKhKBpSRsIhBV35z+O5HWsUkyD912XRHzLT+O8lQFPnFE9XNyeRoAJEeKxnxlpcuGxulJ/eE8DFA9ImF0aWQFCtOucjHpUqUsDnGBFC6nRq2vf8TaOxdY30CftTfVCFQhnqDsSO86Pp8ty4WrgVEzU53gqdoCM2anp+yW7V/0DpkUvbLwbLh5c1vtwgvOFo8vGLNcC58fU5s0OEnux+VRsVDcBxMmws9z35SbOT16JggQp4kVGvaX5MSoafDePAusppetedppmEHiDDJlA637w0d6bOftD9oU7RKT03b7jvVS6F69dpONT7lJrygv2vatN6R+f2/R5n0JgiNeioYJXi8cgdgs2Eiix3n9QdZ4zGf/lhY+UjcJC6RZK/yd00+jfnDleEgENvh+HiILSbDFG9bV15dwb3xgCPFhmicm0wAclXLZOFM2MubBGgFJU3OTTU2OiWpMoSYw+YgHuCmkTzipOvkEZpzOyQnbftvjdrynr+QTxQ0sy9rCBR12ySXnCgZmU3M/nFriEs19b2jQQ+F/dbjU1np9IbFWgEVZaH4Gd48NpbI0zBxqGmk2nvDxVP8Omhgug0AQcYM4iQR86v2bnNR99A0M2+atd4uUQaq665bVet+r19wiS8RXS0utrVtzpahXDh+7mw12b4A4ZCkREwQaCVfC3WKlN7Jq5NqsqdrPffUOVec4NQFfhnnG1LHzAUwI+PhApSipVs3rWfyYDs2Hs+gsGD8bGurTQ6mqIlAb14Ai3gPW7vAI05XGRSnm9zEenDhOPBRlqURD5EReTGM33GSz8SR4hFTY+Jjd++DX7fCRLl+wZOoJ+uZ2ttglF39eboVNiG4OqRnRb2AToYQp7kDykTz8GDEWuTndujR8Ks+vdNWNqJtjXsPPqwyaKnnyqXQRkTqlmrhKpQwsmJy0o929tnX7/TYOUlqctju2rpE41OobvpCGIJudddbH7U//5FTxECOg00ZKuLzirtR6Hd8PX88aB4jm2ZZDz7FBMvfvWF3kwXsfe4UEh/bu3VuqrXNC+CgX7Eecr0IkR+XmExMym1oYhuPy2oxDl/y7KhUrOHWcMjVCVFRYXUOj97mn2vHSk06yPa+9qt1Zm3dql5vgKQESwqaTADEwRvTb4wLuuvdLtnf/4cBIPPjJZmxOe6tdcP5nk0q1qzlSl48TyGIp2k4Vx4CTQ1YV7r6gaYIEPThXsI7R4qBqLL4zV71FWhi+mLVeB/DeA7cibOYgdvT199r4ZNHWb75H/Yll0wXbvmmVmiCu23CHW5NCwbZsWmkNDXnXmJ+loKl4JPl6ucLUnuYTrD2IizQzYgBxJmdRvDNPPri5qFku5eVKdfBv+HR8ReSyfIh058fGramxUZOeQwUa0p/06Kp9Hhw3J6nS2tpSJwkVM77UKl1drWIOvppNIOVo2rAy5s2WVJGkLJkGBwFiJFCH08r4Ut/97p+/+8L/az/6yb8nUoSbMtK5OR2ttnrVlUltclJsov6BvpIrkwImLqC83A4dPmxnnNp7wtEAACAASURBVHGG7d+/P20cFzyk946v0RGkWP1gEHuoOFNI/HQtEtVIL/mCZsIeHh52EAslbmfwuGz5wADACmXhCVt5/Q4bROuvttZWX3WehgJuuOU+cRd57Y5ta62y0q2Gl3T91AaHD0EJAl9POJ14QeMr68kaIBUzu1gWLl2bgRMvOHNyUmkbAR1ADr6NXYOf53TqgZaViTwQ/5bWfEKmODm8BwEOE3m8uodvn3bwowbhYpSsahXxk+ZJ7EjtVhU2PTGu08PvifWik+vTJAI0UmtSBbDujMn68b/92p57/kczJAaB4UXraGu2Sy75vD7PpUhclQq0TeBTZaUNj7hvx2+KXZvJqO88AlG+R8Ap8inFGXwmQ4/QpZ10N8hmlYpXb59iFhhZfhp9ALCSTJlnL37JGihtnLDBgSERSYDAW1oarLd/xB59/DkFfOUZAr4NUr8oSxp7bDanpSW9H03PxAV54ciD7jRRUi7HSTQ6uMz7FZTr5eLMfdtXleRRiBbZaSw8lTAwc0w/1TAV+4FjBweFZXMDkiVFA25iwos2lZVqbyIXl79XLd/noHkg4mpSfuK9i4SNxe4c6utRkIf16Dp2TA+VGKMhjSP3ua/MdEWe2xEoLPBrew7ZV772zRmdPh500ayjvcWuXH6BTtro6LATRhIW7s0gBUXz3G/QpOMABOIWFoyUTGmZ6tmetlIdYFOxpG45/MTTg8c3WVjPnRl4QDXPMx9VNUPjvrzcjh3rsjGJPUyoU+bbz/+HvfTSK/aRD73f3v3OU0QjYw1k/pNiFfcUMKxKsEm2XDSwtLDMo5UGf5KlgTIewZ024z3brlV1TunMLMIgb6CHklgoBDTHjh3TYvE/pp5Ai0XjxLCz0GZXBC1JFMAPj045FZ6XVgl1Q+mivqFBwAbvAZefzhOsA12vnqZHH56f+Gw5phKs3LONnj4Yuhl75fU99qXHv1k6WREftLe32PLLztECtLd1iIeeS+NJXRfeewTpVcM/e7nWI2fSWSwULof75+HREsU4NJ4JQR6bxxnIfqLk+niPSUaCIVPuvQUQKLkmCUgkBlBg5vw+vQVo93FwYNmyOZmRg0VkA7uCd073jJXSGqVpWQHKDDN5S82sHrkHTyAkVbFkfb390jQQykpQeN8XVhYx35yuzrlzZWZZdD6YD+MEYqoxf0TGXCw3HmYrAhHMF5EvEiOcJAKjU0492d58881SH93AgOf1gXpFqzVtUJXykc6yZUEEqkwVrLW1xWe0ChFz009f/sDQoBb7SHePPfjAP5U2bUT3bW3NdulFn1WRgnQHISbwcyhU1Arw+ceOHUkyKv4wdBKS+dRg4YTK8Z6cZMQQCSxZUdI9CjwgvnJxQ0OOeoIjqObgVCf+HXT1oHFFNsFocg5DSTE8658xMjik9+BZzu3stOPHfXgTh0ULCzO5qVkHyOH0mVZtguFjR49plDmvDT4DUARunH/LJRDccWGcxDid8m1J/owXeTQ641cJHjgZHrABsLgfA3L1TkbHwStSmRUxA7B9Bg9wOggOxfhJKhli8PYOyL3gJubPX2D79r2pDbZg/nxh+MyKdxi5rtRdg9sYGR23W7c9YNAdImJnYdpbWuyiiz5tSKgA7iDAFOihIngsVlVOkKoIGIksIi4BSGZCwaSsmUrN+M8RMpqEjjk66vKnWBB6+FlUucBJ9HtqJYIk0Qj6DhNFjSd0YP8+65jToc0caJuzoMo0WkxoZOpNJMbk2rE+nOLWlhbda1hp0kDoYiIfS7K0zMYmvVTMQivwm0hzcxltysF94el7JXdGHo854oHwIVwEJx3zQIAjCDeZsxICVlvrKRraqtTgB4c89ROdyCxXRdsvc9Rm0g8eIgUZ3pub6JzbaYcPHxblGdmSpoZ6uQAsgEaI5SpcqjQ1OdCGFZuQGxoZG7ONm+8RgdHXwQmN7a2ttuLq88TH91nvHpNgTQBWlixZbAf27XV+HTBKmoAVhSQ2PPfOtej+E2DlwxfGSj0Hk+PumvDjoHYcCLlITYigquh+nWMp/AN6mmhkMSTIRBQR2AKqpgDQZ9UyVNC5fd74qSJPYvByaDra2/UssjR8pp5G75fM2uDIoAJ0GEu8J8yg8P8K7p56dGuR3Xrw4EEFVbX5Gk89in7jbAahXgzOZUGSXjy5Ovw4bi4qeMh0RXTP08BN6LSOky56kMNO5f3EdFFXicmcHT18RClQfW2dNOr5u/rFxz0VjNSPhyrAKIk0DY2O2LYvPCwlTPl350xaW3OjXXLp5xL0C7fcIV83s2U66SCF1dV5BYq4MaJ8KWwB4mBdamt9DnwaJYaPnanJ039OwJeIIeOjOvW8P/eIi+G1ZAFh2hXYJa4cr+FeuGZ+TvosskearsWfHEYWaWCwX+VpuI3CM1IbN88QYE15PYcSVDFN04TQGV1OakIt82oi5FAJPN+86vNFOmcOHTzo82KYA0NAQ15NLp9oVujEUzBhARSoaMqykxV5oF7R86Apeu/YYa5ekZFPOnrsiCJUvtfb22Mtra1aALIJ/BI3m2d6hUZhT1hn51zrp6M2je12IMSHApHH8/6UZ9ffsMuZp5hCFSMKWvgVKy5W0aeqslqdfDKfAmO85RndOFJMABBNhEIFKxVgSgBIykBYRH4XtxTxgIK0NJYb2RPuq4Q5CIhCQNEbNORXVW+fKEHEXIkvSnD1/f5kuczJFHKnBReVAtlUgJjyMKXS4hk6stfY3KTAT2BRUvEkm2FThJoZ8ZU4AET1BDKB3ukkFoulQobSq64ulWgx2dJwTaO6XfKjwnJV1TJN1My5cTYIX5HqiVLMOPGmJlmI+JnAG7FyauzwYachQcLg88gI2CREvexyfhfaFXPaBSyl5kJYpFu/8ID0dOS7U8Nlc1O9rVp5hbRfVTYuEJn7MILpwqQCJzIJAKnxca9gaQa96vAuPe4pqVfyWHhlJpWVCb93AcV8jc/VQ+SRe4Eyxu91dnbIiioDSkicov3ETYiN5fyGGfkYZQjQvVKgyXNVYSilnd6945E7VoKNxJcXrmpLimOIWJGFsFayPFUuRhl9jZk7brlKvXOc4qVLl9qBAwf0oMLH4X+5ccyc+wrGfo4IPaJCJohUzQZAlFnNQeUC2MWcgCA6AA719/dpNxK88OVRuqNOXKBvnhrr7JxjXV3H3IRly23JkiXCErhZFonNyBefic/dvOUeG5GQkpyH3qupqd7Wrr7SpqbG1aXLPSxatFjz7tiIPgfOu02HBgls/RipxQsRzHRCuTpew73weQ445YTq4fqQceX7lRWeQxPn8Bp8O6cZ9IyDwCbms0WuTPPwuKbgJuo5UuwhSE7TtLQOafCwIOxU4FETaUqT+VMVRBXDnOrFe9U3Nsq18vmaZJ3z554HUcUdPbBzjRQxyLV5QVSywgfVCfmCkzeskRqqX1d72bWxqVFMj4qqKkGRLc0tQvZiDCe4tZdEvcGClIyM4KSlJ9rhQ4dV8QIQUt2aGfSCdGlxctIlG6Cnpzfx5MgGhtEjVhwRp3B0ZMx23v6Q9Q8RiYsCJ1OPysT2bTeL0/fWWwRxXtIFTSTadnSNBgrH1MmDfeNxj6N6+N6gUVBXb6RGkQcPDwwoiub1vA4iJCDT5Dg8QUfHQjc/3AfPhoWJqppQP4KytBmi2zbiBJ4dC8e/OZgKvtM4E0G4QuSmZCUJ5KIoo98vK7P58+cp8GSj5MBfqiqtd2DA0+aHdq1V349gypERW7xkiXYoH8omqKmu1oPioXd0tCvoIjjgZKjzVcN33Q8TQfN9plRwwVTj8OXKy1nQqry+DyCxZ88emWzmx0RDJic5YFz3847wMYMWc8rNNja3lJo3dfNl5bZ9xwN2uKvXyQoSMTQt/FXLL1B2wIZgOLBSoFT544EQvPo0rH4bGhoUYKLMJevSIdFBrJsjJUq8BKGOlRVyFzx8Veum3NVMjsFBdHcZiCDP8Y9TSd7P9fm8cYUTC/dBAdnUlDaUroHa+6zysdLrRF5l4/D5mH5QVoLzUO5g4XHPXJMscHlWaOgodDYi/3u3XVsEg8YUs2vmz5tnBw4c9FNAwMaAPem1wsVjisSw+1EK/0PEBjXin/NQTznlND0g1J727d9X0ogFHQPpqqqu0ebp6u4qQbPQmzw4rJArwG9pU6UCDuYKCyAs3YpWla8tVZ686FBhd979mO0/1OWroxJrRgu//PLzFXfwu+IMjk/IauH7sFyaDZOrUPZARTIfRJM02I+NxP+AM2wIOAccCj3MfLVP1NB0aDKAvHrfNB9+2qN1FW1SSsufvJ50j4yIwJb3xcosXLhQCKiyIyZWzJ0rF8DPgvdIhM+z4ftYBtaM9+HeOHykbaScvBfumc+m7q9CESqflWzwPuvonOPj2+/ccrWoV1wYaBbzVkgdADHYfZwI9a2rQW/Cautq7Pjxbgcp1EAxba3tbfqgBQsWKdh4Y88eFTuOHDooszw27sI7oF7sUuriUaliUZubW3SiOflAsTwAuO64noiS+Tz52dS3xg25WZ60+x940vbsO5gWHuyaIQaNdv26a7QoAEbsekAkHzgMT5CT4DFKvrbaDhw8YFUpwuZ7nDYHZWDo+hcnU6kX7WRj4x58DvQpI8iD4jHQgGKMmlK8hZnTzmcr4E0NmNQ6cA9YPT6H585z4b6BxTnFfAbIHlYp6FZ8NoeR9YELGVQyFj6wF/7OBuN5UW3kT/7NpuU91QcJzsLCk7bh8BU9TkyKY0dAwwvZUUqAKP8Jqhy1uroal+lqblVRprwypwAMTdr9Bw4odyf9Q/bTOZBOoYrgiL9zs9w0sDCvJwBbtHCRHTh8SNaAYKmXacpJDIFNwyaorW9Q1B9AEzoCTz/zPfvliy95mqfGTZMcyoqrL07TrEflQg4c2K8HXFvr0Ce+kWvp7nUixwAQKrl6UgHhZHGSCHjD9NfXU2MYkHii/Pi0y6SjOQdbloVXrp1m6bCQPF/undezCByCUPrgOfzud7+zBQsW6FnPnz9fr6V3QSc1MaJwURS9+OJ1In3W0z3r2YQDaTmBTcIGxh0yZkNw0gX+5HL23ve+1379619bZsu6C4oEZUCP+CwWFFRNAgIELUmNkg/yC3YVB6/aHbXGhkZbcuIJYsP88ze+obo2P+fimhubBLm+/oeXtePnzJ3ndeK2NkXtdXWgdAM68ShO8XB5aCwOzX0e3abOWRWHYOb4BGeEijiNVblK+9mvfmfPfOP7LiuuWINWq1q74pJzlCU49s/UKm8I5YuNRHDpKaW3j+VpkEilUzYAnT/4YQ1CTNOriYNA2PgdlULTtKmY8Z4rc4YyMDCmVmlwKnhFFB9FG5nuoSGdcmIfPjMCOw4SGEfEFqxFYChYTDYk+sNSJEupM5uGU87mYkPx5VIxno3xfKlUCrm7beMVRXWKpKiWF7vSlHetjAwNe5cpxY3UKDk6NqICBf6VEmVXT7ebqrq6ks/B17zx2uu2aNEi6zp8QAtOVK+IHV6czJM3aipTqHH/xRc7GdE/brC+vtF3bOpmxdqoKpZQLJC+3a+/Zffc94SnYEp1WPgaO//zn9am6uvrtWUnL7O+fvrwHH3ErXCyiFmGR3zYMf0vge4pVshmlbLxoFg0ngMPlX+THeCKGuvqU97tDJ3pCWrt1Md94pboWKl3TmlYCqSxKirjJiYQ78l990GBIzDDNaFUUkWxaqbeLiJnoWDHu7ttlIENCbPn+fNe2igJ/Yu/x/eV7ma8Uph59I71iuoxXYJqCVwgJPb3loR5hwaH/lPbNDm8LECuPOXUTvUhuuehMsWZhwKGT7GGUFC4dch0UCiYnrZFixcrTeRm65qa/T114jw7EFN3xDdepEDUrQnIGpo8P+W9D3X12l13f9EFHBLwAfNlw4YV1tfnwBInWxTwXKVONy6GB0KARCmY6BkiZXtHux3Yu89bk2ZF3XFqA6lkk6qZos6DUfRllXINDft9oGeT3Bvv5QIJ7vOVMZGTj4zIDQR0G3FMUNtb2to9xUaGvabG2tpaUg9jTgeJg8nPAbckHZtIGuSZpGz+5RtKI1nT9agY9MW7bxQDh2I+vp03Y4FIT6Sn1tMrvx4dMyw6YAonulDEV8OQpeFwyoZh7wD0JNVHTKxGh4F5T3jk76bc+fhcKEFOV1e3zV20yF5/7TVra2lNPpLFB+BgFq0PG3D2al4na2IqjdwqFm1wrGDbdz7glOM0mQGLtOLai8TKxczjUvbt22fz5813AEO9Zk5oyDGWVFQpD8gIpvCVjkm4v44giWcDs1gyY2lapSt8AvBM6V4HBgZF/Y7TzObGYp104ol28JCPMvMEpCjAiwBOzzxZADbHsmXL7ODhIzLdYPRsVKTZOfEgkDzXqCdESqjq33RBPzv99NPlPl555VWflVeeJlNZRplY5skHNhWZ3X5w337VdwFROPljI/gCKMyubQe9mWIGN8eFUd3iQo8cPqIFBIgJuhTpAj9jgUhH4KHNLlQM0ueeWLv4IoI790e0ZdUpz/Sghn5296XkufhbfBQ3XyEKlgrRNjA0bHfc+VjqX/dCECfkkkv/0UuUkC2ItDUPjyjegy2weqwHWDhVPRYo6GROpXZBBixE4ApE1ELIcj7eFGtB4DU+MaZshw3Ha7B6vI4xqd3Hj5fMNRaD58f7RyoWMK2eX3m5pmxj6mlYIZClfqLIvTwj9PGV3X9Q8ByQeBworFkmETKGhgeEFH70b/5ve+WVPyjOwRKQdqq6+aV7b1JExFA+ThW+Avwa0uNbb71V0nalGAIRAL8DnYoNwEVxkpwckU8ivFm9BynOosULhVcP9PVrE4AVYKIo1/Ilc79okS4KdM3fF1yd0qVTukh9hEgBJKX5N/hsGh85daSU5RU523TLXV7ISHAm17N8+ee1gQjIdJLLoHwPWVNrs9OnoECNg3Hn9XnBrxNil8yyePXFokypQ8KO1g0yb0aTKpzsSNArOLYwYVXM8ZNoErJsY4oTsKq4Ew1KTPIuXFdYPtfZcUAM9yRO/8iwm+k0hgW1UVf28InaYY3405FIpnJ6O/fChfM1WetY93H78Ic/JGyGQ0j8w3VnvnzfzZpJozr05KTKosLAJ6EF9WsRPQqusDmdXjsHBZLPVOHAmzD49wknnKBAqm+AzeCFUzYF74OvB3fHPNU3NmjHHj58SJuFgUR8fmDtRNzk69wQn8vCn3rqyVrY3/3mt7ppzLI49pr5WrCtux71lqfU5oiPX778ApueZpqFyarMaW93WlW6J6BZTljQjtU7l+bJKU1i/HdquCC1YvHJrUVSUarkEjBu9oFq6eLxfJ8TqxSO/rnBQVGnAaWcdeMkFlkVJlkeOpKmZHvAhyHTJkqoJZ/rC+uEjEA0eU3w6LznYcqytLEVCiLWiOGUMd1zjHANelbm649tK2LKtFBJBgSTD/qEmYcASSBDdMzDBDtXVwupwZDj95wW0gsRKnI523dgv33gAx+wg0otZtIJV7V2UQNep+ieIcOkbYqUY+eip+NdIJHiUUNXIwUnPJWBMeH1TU1Ka7bufMS5ZIlszLVecMFnLFdZptFkkkPNuKIXlTjvGBrzGnU265y3JIyAb4+/q+w5ewxZDERQT2G9FpJoHXEjVdVE+vBytNKzEa9A8miF5kFrS6eeXFs+e9QXvKWlKU3HTouMRKoCYub8EARSLPLSclTrWFzAL1Gp4RFMOL2d95Vu0ZQHkVFj8EOTdSIGIAzUIC5q6dIThfkeO9ZtrW2tCqzA6WUVYp5qIuydcMJJtm/vXsGMXr50rRwujJtvbW6Rn2GYMKeEoGg2jEjMgCUQSlbFn34CeWjE54HbRx09KmMsWrQIEfw1NzfZhk33KkZJDWtWna+0Ky+/yArTY3bayafZ7t27dQ3KsS2NRkuEC31+0ujFtQB98llt7e22f98+neQ4XeIMJhPPQgCB4sJefWW38nEYRF4hdE49G5WF4P34s7Ozs4QlsKHkgoRquuVUrj86at3dXcIgnBQCv69OmxP8JBRLmNHHsw7Xi/VlMxIL0a0r2HZkLE3ldqSRz+E6M4/fs0GmvhJcuhzpLm+KBIXjwR/rOip8ndmsPCA8F5RnLrK3p09+n5vid1h4/mRXcZMEJVJpSpuKG+Xhc+EgVSBp+HdV2sYci4cRo9NS7Qxebgy3EOlUwKaoSjj6VWZz5nTY6ut3ajChu+FpKUlcdvH5lqs0Wzhvod4Hl8P/pHf4dnw+zJuu7m49JK7t8KFDRrDLn+oM8qPq6Bh074YGReKwd3SKUtqUKy8T0tjS1KDnxGZQYWaqIFOvAk4isi5e7OVhfs5zBDDzlBCh5xG5ymgSZfGpYbiuDfGFN65geTvnzdV1URmlkMbJ5/V8Vv+gB4gEyzzv/v5eXZMX0fos8/hd16uLmh1K/k6q45Qd998hPBQSH1zsgUOH9YFwvoQNDw9qIXmo3CSRrgMLznFTE0SxqEieDwU7P+2005ReschRueJ3Gpsa9CAYMBiVpYghlPfWeQziIIr3qhFNf/FL37Lu3gGN5NCEiVzOVq+63MYV2HlxRtBdkl/DuolnNz5uy04+WYEsmwMkrSTHopGiruilzCXBrYoLkmvUYWDTV5QLJm2sdx4iETZgEQ9atXTIGslP63SDDPb36Rr4t/x91nsTCaSPH+9RysnP+CKdw18oOG1qVpoLMQX2sFrNAvXLlidhSA9EuTbdV1LRBK+ZN3++Zb5453qNJglcmoALKBUT3N8/oMUMhg5+ROVWsWkdcePGYZLyxckFatzz+htJF29cpr2hsUkLD6QIGkdEzOsw4SwqlTEu3OFFpx+B2Olk5fOCH3kdOW0ENjz8qPVjcVj4o909CmYwr6SUVy+/wIY0r86HJQDv8loRQFP/GVbjlFNOsV/+8pfaLIEQirac0sj4XnDxFBWnDhkwdbFsUutXZwdwdFdpkUOdCnUQUctQDUsR/rGuY7oHClq8jnEr/Ly7p8eWLVuqg6EYJCFydQlt1ABFla3x/04Jw1KiJ3Dg4EEVYYjRgqcYAR0HD26j+PWP3HZdkXIlUXx0XvDQBgcGBXzgD+YBeowSJdYpNaqpd9UMomi1W/X3yULIVShSLZeZyedrZaZggAqwSDNiRsZGZbpY6JNOOslee+01ZQQUQyicvP766+n389ooLHy4iKAzcVNBGmHzPfH179qbbx0QCdPVovK2/LKzrTA2ac0tDTrZCxYutD1vvKGS6FuJ78/G5CF55uINCxFb8D3BrhMTdvKyZfby7t0lBg3Xz7VF0AYjh40xt7ND18/p1eZJaKHLrngJl3QVi7d37z4vswJIqWbP73gAzPOL6hqDk72+79mAtHlF1/LFfdfpp9vLL79sdfUNSuUIltn9vCYsYxwULI827m03XV6UGTSmOfbLj0SPHHktfie6QgFYSLWYncb38IEnnniiHT54wJYuPUk3jAkiAkdJGk1WPmTu/Hm6gFdf+YNuCBkx0g0elDhwSVQAHxQRaNCTeFj8bgR4InqmICjydn722JPP2t69B0XChEgBVezq5edq4Wtq/DMwr4J5wctpDKUMevRoKSJHn0YpHOzXRMNS/AOBIaGSLBTXwCmlhkA0r5gEhJD4ZWjAq4h5ytfHpQg2o28LXa22VE2TC1Cw6ILIuFYWnqZLDpqKZJmM+A5Y2qVLl1lbW7v9fvfLugZa0kBbeR8KbFgv6OgLFsy3ffv26nPASThYUeDRCFa1UG25poheLaeeKD4wXo0T08NCCWtMgYMP55vWCBE1WKZmymmEjxgSkPdZsyBi4qGlliWoSywE9fz6hnpZADB3AidGjfUPDBr1gNjpgfJhbQQBq03awRlAkGh0ZDHxo2WZCvvmd79vv3zxZXHKYdYCb1512XmWLfrkCLmmRElSPSHx491v+8PgRPGemHwCOSzNbJ8vcIh2KLV5eZ4PM1fl5rExzXg7uH+fglI2GP/GXLNp2GQqG6fBSNGHCLuI9q7ow2NDAYodOHjImpuaSvGGqF+ogNBJm2TbyPe5D96bTIwdxqYjHti/392nGFKDrunPa5llK32ie29dUSSvFfm+ucWOHT0s8QB2fwj1xWkTzxwevSpzMzIbUIx54+a2ZlGCqem3i5yRZqAxpntoUGkh/vTAoYMGpRvMnx3Z1wfu7L43SrpRP2YjCeYcn3SZlcRa5XNYiGE06spy9h8vvmTf/+G/C/yAZ1dbU2Vnf+aTlq9w5kyAUUDLasdGIjU1kODmRPzUTLnUHpZ8uNQvEnE0zCaY++EjR5KlchYwGQInv6ba4wi+x/1Qv4+NvGjRQuH/PEOuHatIDYMNzgKxgaLMirVgERU/JJYubOawklw7B4vf4X6Ih/hZBIsE0Pwu38NKidUEIol0HPf44PbVAnCii4P55OTumOkaATW0D3t0yf+cAhC81994w1E3RBCmXU6EDhnBqML3qyxfjVBCmTU1NSp9ES2bnH98rCRH4qVCJk95vRlfxHuRu3reXukl09QCxabDrImGVVll+/fvE3y7+4299vgTT0u8IauFr7ZLzv+MlaXxKVTBcC/CABI/X5Tkujo7dOigTjlwJ1aOzIbXhK4di0MPH0GbyItJ5NDr626psHJsRip8AEsLFiy03/zmRS3k29/+dqV6eu8JRBXrFZSxIKR2xC08B6hgArTGx/VZvAfvSdPo2962xPa8tTfFOs5o4pl4EDolCBpLRPEMXOOll36n5xcnPdwGyqWsRWbbugvVUEEKhQlBQlMPRHnhuI1PTAlp4jXC4EGOxD33Sc+8uQr7CdQJoqAujLZdSYVOKpI8cuSwAsXDR48IyGCnc4qJKagtc8qxKjRa8jvisA8Oq+yI9RBF+m1L7K29e62hrk6Vw9bmNqVik9Nltv1OKnSwSgtWV1NtV1z0Wf6hoBKzPFtiFPOIxUEMghNI8Id5F0rZ1CQSBEN8hQam6pznw4OJPu5ZTrOwWAAABvFJREFUTGDvIHROBfCYJEqgRNtsXII6CkFtczpkesEh+JMvTj6nSzP3VCHEZ494Kq1NjwrYkAYl8jwbG73rlWfMurBxJLyUAB1laalbCYvgKGWSgU+/l9l+/cVFpLkwt21trfIvqnc3NGiXAtzQphMa7ZxoatZAlbBOojLEQ+ADeRBcAOkaqYMHRpzgCQWCwqKtKL5Z+G8CSJBCHoT8N0SDnm6dlob6Rj3gI4eRP81aY1uL3r/ryFH9WZUDSCmz8SmzGzdvV9Mg9KeafM4uu+AzVsyWWbWUpt2PB4YOTCuzy8ad1TDJ94Jq3tFBQ4e7lEhf6d1z7MERShaH9yBd4/5h33JdsSFU+yZAG5sUlgDKScyDBaFphA2BWed5UzvH2vL5xFguFU9KPKxaw/HeHnvnO9+pcSxYXiy1KqkpLS5RvmYri6eFn03OEPSNjxdAAfOSC4S7pTbfKevp7VGKBuEShA5fGcIIAV2qNJoeaHdXl0622q5BqdTsT8BHKbU+FS/qrLe/z04++WQtPr/PotTVNSifR6eGWvKRw4fTA3YtWKLd4eFxa2pDdRN/6Pg7o8zkGianbMfOB2xkytUr3vOed9mH/sf7LFfmvWlsnkgh2XD8OzIIrAlLywOONDFSOR4498TrMZEshuoMtEez4JWV+v67z3iHDg3AixdVvPERq4e76pw7T344MqTFixfJXfG7x4/3yvJkyp2AEvgIm4nMig5dxz8G9WwCKY0iFu3nsjKTE3JP3O873vEOcfkWzsciHJAb4Xq4LjZV5s7NVxX5UHwPPogTTQ15/779DhXWNyilU5ExhgmlZgF2rwgEaUQJf8eEE8k6ScE7cpyPRp8d+Wmda8tHg37C9slJA1o8/YwzlGcTmLS3z9HD7ek5btlsTvPtcQ9DQyPCEQBlvI5g1j80Zt954Yc2p6PFFi5ot5amZsunFqpAwBSApdZh3pdNRZFHRNNUYAnXFVg69+DFEidYsrD4V96Lf3Pdbz91qcz1q6++6n15GhA8LkugBpMCJW+v2EEqpTNYm3loWEr7YskyRSs9D16HYASvI4/n8/k8ov5onuBzvf89uIbetctXXC8CDX64YA6TXeS9d45OGrUhJ1YoJowHQu7HLzQ1tSQz5PNWPJhw3pZy/ELBWaTqb3Mcm9ewu/g5fx8ZGnS2SL5G3ZpUjCIHp3BAIAN4I1p1olmJk1dWJloWppj3amlpSxOovd9eqhaa+Ybahte6OXHeIQOciYS3B5R8EcCSe3tFi8qYVx65F+IINgHXHac+ImbftB4xhzvq7JxnR48csSVvW2y/+MUvbPHCBXpf5upQZqbRI049+Ln4c5U5mzOnU00msHZEBqFRNV+tE8n6+Wn2AktM447NiushnuF68f1oBcxUL735MrKgzg5Suv26bz4jJGe4Rlk6miZZdGrF+DOUKKKYQD66YP5CmXmfHu2Nj/gYL0WaokgCQ1XUph0z5mHGqWEx0cKXJhEQYxrnIXp2InZwgbyO3yO9w6wRaFEDj5vmmubNW6A5LgRAMHz5OYvOaaUbd+68ufbS715S12N9nevToLXHfYHaqfxb6uwdV0ApBm0qnvCQhN+ndIx74Wfcc4g68vv4V1q3+KKoJe5bf58CrUWLF9jvX/q9vfvd77Gf//znej9cBfcWamCSXU2jzvH1WAbFRF1erGlqbhRtvafHadFhBaiJ4PP5fK6ntbU9PfdpweE8R3EUYCtPeqDKCef9sTqk6/xcXUNP3HdzkZSGU8cNR3QI4MIJoFIlKtE0rcXO62bXExEvmDvPiQzlTg6I4gUXyqnhRr1Jo09/Bh4gaDhNV+CU4tvhe+MigpoEygYqxfu4C6AChabulDZM6NFyoufPW2S7//BqqVWrrtaFF+hY5T0nJrwVKXJZpoY5ROqyZgI2YNGWO9jBZ6jXL6lhuTy74+xBjOT3+Z8TxLOb0+6Wq7mlMal4e4eu9/oPG2JEFLJACjHv3Bdw9euvv6YYQPFKuReX2Ozx/vxJ3ULo3OiwGik62zt0kHg9hTUsAxuUplfiJgFrYfKnJ62ttc06OjqV4jmHcdoyO2+6rAhIAbAC3iu0h2pRahkGWXPFZ4CC2pIejqDMcl8U/G5UzXhg7PJgfCiKT6adm1C78+SE0LtIMXpT+dWnS7nsGj8DSJJ4YqI6QzKMmXFhJicnaSHK+/yY9OCERasbZkhB5Eu//40eEE8rfDrXiRuJiN3h6Ua5HDD7mKnnCCSl0y69ln/zu17r9tHoqrZJ+AGk02vkyIuhvBF1dgQLuIbe4z0lxhKHQSVwMZCnbJA6SNKpjYIQh6e52Z/HokULlAIDu/K5R7uO6WBSyeTZxrWRfkd8BTfQp0zOVDsJ+v4/WJZZZ4vk0WIAAAAASUVORK5CYII="/>
+        <xdr:cNvPr id="18" name="AutoShape 8" descr="data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAH4AAACpCAYAAADtGIkfAAAgAElEQVR4Xoy9B5xkZZU+/NxbuarzdE9ghmECQ85REBQURER0EcOiIobVNbCGxV1Zlb9gWHPcNaC7ZteAeV0TuigrigTJGSaHzqm64q177/d7nvO+1TXjhq+VX/d0V9269z3vSc95znmDeM8v0iBXBPIFdLIV5MpHQl9paN//l6+p6Qn84qYb8fh0C/ONCHESIE6AqN1BHMdot9tI2hHSJMHfvuBsTE9PYcOGQxBkAoRpVt8DAGEYIpfLIo4TRFEbaQoEQaD/0jTVf/yZX9lsBplMFu12S6/zd2l/D9BqNTE0NKT3RFEH/HUripDJZPQzX5MkMVqtNjKZUNfgNYMgRBxFyOfzem8ul0MnjpDV++xT2lEbhXxePydJ0l2ZJOH92bWrCwsYHBxEgtieIYXWIghD7NyxA+vWrdP7/LNpqZEgRYQw5WcFuq+7H92JL/7oN4iRQavdRJQESHkdvp43zXtAqPsIwoz9Lg20hvy8OE3sd0kHnVYdmRR4/TlrsGHzIShmQwSd3T9Lg3wJcaEfmf71CDH8/1vwSGPc9F+/wV1b92GiGqERUeApkjhFq9XSwqdRB5kwwNUveZoWh/cSRTEenmjhqIMKKOQLXaF4IXMhuRm8wCmYTifWElEI2awJXgtoa6DXc9GiKNLfC4WCNh5/1+509Bn+q9PpIAxto/jP4PspeL6Oi1kqlbRBHn74IQwODWHVylW6Lu+hdyPaz3avS0tVlApF/RxmA91Txv2N10y4iXs2DBckoYJELQk+ifgwKTpJipmFRWzdtRdxkMFCE/jDn+7DUjOVUP3GS4MM78Z9PpAm/HsCrh+3kjYcYsSthhTwjecdjPUb16GUzyFo7fx5GlQGkR1ZiQSjyCQVJNSKNEQm5NI0uL1thdMiEPI7F8BWvV6r4ds//TkeH6+hHrURdfiB1LZI/4UIkEljvPXF5yFjSotWs45H907hsINWI05iLTQXmQu2YsUKUDBczGazgUKhqAWnJdDu5mJJw/zC2kW9heDDNptNXWdpaUmay/fZxuB/QCehZYm618tns3p/o9FAuVzWzybkRNeQ5gQBqtUq5mZntaEP3XIo+vv69DfejwkgQODuLUk67r6cNtIGJAnSBJifn9dreW96T5ggE4bI5mzT8TPnFmt4+PHtKA8MYs/EHAJa5CTA7Xc/iKUm7UkHtJeUU5gmiCmrGIhiW0d+ju4rTZC0KcMUf/XkMRx+xCbk+drFvb9Pk2I/qs0YhTiDXHMJmaSJfK6KrKxHKjMVZFPE5RFkBs+QMJfVLcUvf30jbn1sHLO1lsx9p5NIeFqUToww6eDvXnweb1M3045byCY5IJcijrzJ5AImKBaLWlgKkAvDf/dqqjf5XtDalE7j+Z2fy+sMDAxIUDTdFDq3MDfP0lJNz5TPF2SVKGhqJc0rtYXfqfVmIRJtBm+WeV95aovbQP5e+Ll8favdRl5uqI1s1txDQK2UVTBLwbXhpvPmWvcWxLrHMEy10WdmZvD49p1otGNkiyXsGp9F3GohXwTma21Umxk8+NhWtOIYowPDWDM6gHse2wagiKhjG5pOkMrEfyNqydS//IxRHH3sYcjRDV3zgY+klUoFU1NTyKQBchmglC9goD+LF55/LIbzixJ8JsigU8gju/J8hCltdtC1s61OHf/ybzdgz3yMatsEyC9qHn/OJAmuvuxp2Ll3L7Zt3YrNmzfioDVrzBXQLIY0uSZe+vp220wuzTW/+Jo4AIpJqof1LoEbI5PLaYNMTU3KHVTKJUTtSIKnkVpcXESYzWgD+c1CM9hstmTJKHh/v7wHCl4mmsIPAyzMzyPP+wiARqOJUqko7XdbH7EzqYVsQZvOW7Ukjc2sh1kkaYIwzwfMShHA2CPNIU4jPV8my+vxirYpOnGMhx57FAky+nwa93VrViMMUuwen8DCUoRCuSLXOr57CusPGcbCUoIbb3scsbM0iUx+jDjifXTQhyVcevpBOP7YI5Cjdfra93+cTk5OIZvPYXF2Dq1WHZ1mC83aEi668Ew8ZRMvkKATtVBZuw6obAJwsAu2nLTSGD//9S9x1+PjmKjTZ1mA4bUvm6b4+xedi3sffACDAwOYm52RgLm7qZGjoysUsMnP0i8FAbgZzbS7YCbsIBMtIc1YDOKDuXyxoJ/r9Tqq1UWUSyXEHXMfaWwWhM9GQVNb+RkdBXctFPMFZw32DyYtwMogl8mgVltCJpuRsKn9vGfeEy0X/TEFz/9nwxw6nagr+JSCp6Zn6EZChNkYxSjB1h/+AgPnn4MiN5CWzwJDfiaFVqvVkM/lUGs3MTs7q/UqlQoI6Q6RYseOPRgaGcHs4iJ27NiNeq2N4VWjCKI2vvrLe+UAJHSa+JhrEKPTbmEk38alpx2E4449HJk0QfCOD34kzYQZNFtNLRhVr6+QRy7I4PynHI/jBsaRBDk020sY3rQZcaUf2cxJ7qadEQ5Mw7/89e/gvskFNNsddCLz9RRAFhHeetkzcMedt6Ovrw+7duzEMcccI+HXanUJmQLx36npWgi3CWgRGlOPopx+G8mKd7hg0KL+TC4rTeQmu+22P+KUk09BTjEBfawFiabRAcplBmyJgj0KfqBc0bVCxg30i4r/GEMkev4AKVrtlhbcgsUIWZnkEI12w3Q0yaGDBKWcuRMf/EnwykKyCOlKqNWdNh79yBew+nUv12sz2by0ks/HTfOlL/4Lzj77LKxcOYpyJY9cJq+sIuq0XWzEOCdFua+CyalJHLJ2LRYbEXbu2YeJyVk8vGMav3lwL8K4DoQ5cylUgqiDVaU2XnTWRmzZvB6gqX/Lu96tfddxfpVBRtxsYMuG9TjkkEOwAtM47pAYzVaKVUccDpQqCDIbkIYruhE1nODrrSo+8cUfYu98FREFrwAjQSGu400vfibuvudupTrc0f19/RI0NZWawZ0+NjaKYrHkAjgL5LiQXPBcPo9Mu4qwOOjMv5QQoYvwd+zYidnZGQwPDWPzpk363Hq9oVSNLoAmPJfLY/v2bZhfXER/fz+2bNxk6ZpiAKDdifDJb/wSrX33YsXgEAYH+7VBR8dGkQYBRkZG5AYp+HZswhifGUchl8FAedRlCpa5cHEVIHJzcrMkKZoZoDYxhU6mgAwySNKONhQ3CTfiXXfejqOOOlKbJJ/PoL/Sp+C31WxZzBGYBeOO4vfFhSrmag1MTM4pGJycmMSP/vgomkwL40Qug66FmdWmkSxedPZGrD94NeK4jeA1V70t7fo4mp2UMVeMSy65CFOT0+jEAR579HE866zNOOWofgSFQYSVAoLcJgTpMJIgRqCcn0Jq45Zbb8cPb74X1VaLKaQWYTDTxute+EzUmnVF6ktVi7Z37NiBww8/HIWCBWC9QqcGc+GoEbx2LhMqIOPvvannxmCEzvu/7757sbhYVZ59+mmn6TWNVltWI+lESs8ovPvvu0+awLs9+sgjZL658crlCh7cuQ8f/Pb9uPJpwxgaGMTu3bt0X6vXrMGGTRtldnPZnEy/rpsk+PUTX8KmwnOwbk0/skFemRAjfL6v2WigzRRRAVyAb/3bN7B+06FoNprIFYq63pFHHYn60pI28ezsJFaMjiBIEzA2NHdYQLvTRtzpoES3FobIZ/Nah4WFRSzUm3j0iZ2oVhuoN5r4/UO7MbOUIHJ5fNrpIG5GOPfoEZx34joMDw8giSMEL3/jW1Lmf0p5GNgAGKoU8IJLn4PFhTrjEH3Iw48+imIY4ZXPPQKVTBXIZpDk1yE3cjLSJI8gJKDCuH0JH/rcd7BzugFaKKYTo6UAr7rk6Wi2qIFZmTVqH687NzdrQVmlguFh+m8LvJjSTExMaAE3bNigTKJSKTvfYj6RWkCgghbhN7/5DdasWYMjDj9cWsznec+n78RVf30csi7Fmp6dxbZt2+S7+d7jjz3GNkFAN1DGzp3bsXdqHpkkUrBLa8QgkYIfWbFC1oqWwjIASxt/PfV5bK6eg77RMdTm5pANs9rU3EzNVgsbN2xQlL5z507s2bsX+UJZcU2xVEa+kMehhx6K+lJVlmmxOodyOY8iQSKmtKHhE8wQCsUC6JK56bKZrCxBbamBbbv2YGJmEVGUYGZuHg/smsPjuxgQZtGJmR01iTzh5ecfipMPX60MJqHGv/T1f5MqCGDixwgzAM44+TgcfdTh+NOf7kMUmy9dvWY1JidnMTG1B1f+xVEYqt2PTjNC/3FPQWbkFAQMurjL0EBUn8XVn/oZlhqUfILNa4bx/HNP1s3uZ6eVH0vWWkjmt6NjY2g06hgfn8CePXtw+umnC/EbHRntWgYfnevtYYg/3vZH7Nu3D+vXr8eJJ5wgMyNrkBIPyCKJIgnxlj/8QUIblhkfxNFHHWnoYpxICLV6DVMzM6gtLEqo2VxOm4jBICP7NavXoFwpy6r4lOy+Jx7AVP4OtKt1HDN4EVavXG2pXauFdquFSl+ffvaYAnEOC+kYzWcl8Fp1Ud/n52cQZlJUaJ06bX3G4OAACnlmL4w5LPenJSDwMzk9h30T01hqJVhcrGF8cgq3P7wLaVBEGrcw2D+ING6inM/gvFPWY/3YANI4EpoXvPi1b0gVfSaxfEIuCHDB08/C6NAQaswj832YmJzA1MQEVq1cqZ3M6PySsw7HxuqvcfBp5wLZPLKrTgXKa5nEIY2X8MjjM/j4N25Gp5PijKNW45xTjrHgURmmhyzNT/svRvaz83PSKm4ELiDTNAaAK0dHLUVzUK5/D9Gr399yCwYG++X3DtuyRWkU79NchWUY//7vP0EUd1Cv1zDYP4CnPOUpyiYoeCKJDPwWFxcU+XNDcSP4qJt4ALV21SoKNZR18HDw4vwCwlIOeRCCphu2TdeOLYAsl/oUv/B9yjSE5Pn9bz8060tKjaNmA5kcIe+m5FEp5DA6MqwUVprPjZjNal0InO0dn8DiUh3bd41jZmZOIE0rTvDYIw+jkxIW5/qmmJlbxBuveC5WDPUjAP1vB8FLXnsl41kkxMi5C9MYFzz9yRjs68PIyoPw3e//BzZs2IhDN29CjYjS3Bymp/ZhamoGpx67BRcdsYS+0RGkURbZkTUIhtfL58edFn5ww0+wYwY49YQTsfagtUhSQqghgh7s3YMjFBQfqMHswqVhtADUFP5+zSoPmdqiefDE49U/+tEP8OxnPxv5XFYC88ieoYIJvvWtb6HWaMjMjgwN41nPehYKhZwEz6zANhtNo48tLLjsBYxmZmdRKpYk+IWFeW20pVYN/YVBBGmbS4rQSbUZtXXtSrlProvXYXyTybEWYICPNF/+nJrM7AIIMwSRAqFrvH4hl0Olr4yQbq3TkQvqRJHwiUa7hXY7xsTMLDpxCjrq3Xt2Y+v2HXh8zzxajRAnHbcF//mHu3DVZWdhzdgIQOyAgn/xq/86ZSrD3cE8cmSwgjNOPVFARTabx969M7jngYfR11/BYYceqhvs6yvj8ccex/S+Pdi0biVe+pQKiuWKHqCZFtC3+kiAaU4c4QvfugWnn36StJU5pfd/HrmSBXA4O39eqFZdsGXQKYMvoW8Cd3LL5qHnJ+HXjJwd2KN0zL2Wf7vpppvw2GOPKTikmTzuuOOwZcsW9Pf3KY1lbYGL3GzWXexBvD/X3aCG1IUuj7eoPopalm5mrEbA/6TRLjefXZiXxq8YGtFmaneIT1hsYM/sN1WAbIbWKVQAawheiDyBtEIO5WIBhUoRGVqiqI09u3ejVmtYLYM+P8xgYWlJiCQ3RL3Zxt7xSXzz5/diurpEDBdRJ8FVzz0MGzYejBzRUwr+Ra96dUp/YVqS4JgjDsWmQw6SqcvnCgizBfz+1rtRb9RQUjCyCZVyUbs+G7SRaczj2KE9GB4cRJhnKpZFFORRXrEJIQpYbLewb5GbyBbS4NP9v3o1a3xy0upVSYKxsTEtpNA9p+W9xRvTGHst/feTzzijK4ReTb355pu18ShcCpzvocaMrliJhx95GIcddqhuiJAufa3/UnlC92z+la7QinCEf1vaXNS6YqHgAB3TYH72vfc/jF07d+Jp55wrX01s3XCJ5Y3iP4eCp0JRcQw5zCAfpig6wRcrRYT5HJJ2C1sffxyZXEHK4HEAru327dsFz/J384s1XPtPN6Da7iCKAuTTCK89fz0OPWIL8gqeawhe/TdvTGlOozhCmMQ46fijEMcRWq7QsXbtwSoQ0Fc1G3Xcc89d2gAEYsaGB3F05hEUC8BA/wDy5SKCXB5BNod6M8Dw6AYEuT5MN/Nox3l0gixCpEKOzF57HIi733zgdR/5uNIyBmMffc81KBWLLnWCgJCudXDYAS/zuc9dj5e//Ar5P7+JPOwqH9qkSWzJT1NYvHeLzjN44RWvxre+8gUhY9RMvzFlkVTBo3ZyMwQy3VbetZ/9a7278huR36uNJv54+20487TT9Fr/5QtNvJ6hkgmymUSCzGWySv0YzdNjlfM5rXWhUkCmkEentqQUOFfIo9mIUHHPkMmwfgCMj09qA9JFvulD30A7YqU0QSbo4BXnrMfhmw9W4Kilv/B5z025GOvWrlVAcfDa1ejvryh9mp2bRZxE6BCISc2sEKTsL1eUfo0M9ePQ1h0Y6K8oTy6UiwhzRJtyCIoVtNopBobXIghLePvHb8DehTb+8tLn4vgjN5omOcxbwhKgkeA1b/8AOiHTwgD/dPWVCAPnHhJfj/eVQds8fMhf//o/8bznXaJrMrWzwoyle94ieKEIPnUC5ee+7K+vxJev/2cBLMTK9xOig1It9bCSrxe2TwO9Zel1XYK4EeC+B+7HkVu2KENYtnQs1tiuN+g3RiFv0XpWpjsE91kuG0jwMvXlAggQRPUlaXa1XsPw0KiCPX6x8ENwaXpmBq1mW3HYWz78TTRbHcRRG/l8gsvPXodNB6/D8KALkJ/z/EvTgcE+HLppA4rFAlaODQk0YJCkuncUK9qtLi65Wm+iXDKfy2NkcAibc7sxEFRRYP7JSleGwVUWGZZTcwV00gwKfSMIikO4/LrvoFGrIwlYnkww2NePjetW44Lzn4Yth6zDJ6//Mh7dPQ7kCtoI1175SgyVgLjREkKnyJZAKgkU4H1VMbhiGPNzCxjq7/szF+Kj+t4/eEFp6VPgjf/w//Cpj7wfiCPVnVi4sYoagSl7J7+FQQatqOW0ny9nqhjYexwxQ9kRU9ogRKsd4Ikd2+Q2ezV++V6MEEIrUypmtFnzJEi4cnM+E5hlLRaQKxPCjtGq1bFt+3ZkCzlQy5tNuqYsgjCLUqmCMJNDNpfFtq3b8I4PfQHVdgYED1fkU1xw8lqs33AQBomM8tkvu+Kl6dp1q7FuzRoMDvQpcFMli/wOmjWmBQxsmg3ML8wrNWm1Y5nKfBhg3Wg/VlbvRLaYRblS0aLxBmju+RC5Yh+QZJAvD2O82Ye//8x/oBU1EGYI+ph5lwYSnQpyAjYCFm8yKY5auwrFTIJmdQnPe9bTtdkCvjYT4t0f+xz27NmNv7jwAlx0wTnIWu7lavWe1cPCiVUAewUuoVNoCPG17/8HfnrLHei0G8jEEforZRxzxGY8/aln47CN683KxTHe+9FP4pqr3uSw9VAFIC6gIfIGTfOzmOb9/k/34f7Hd+D8M5+EjesZpyxXLL3lYebCzUXLUSnnpGw5MpPCjKGY2UD5e4WxVoUwbQeNpSoeeuRhlPv6FHizFkJLiyCHThRjaHgEYdYRWDJZdBAik3Z0j1a0S5D4MvGr/+av0vUHr8f61atlvivlfJd+ZP7NLsSImNt7sbqoaJVwJMuEQ5UK1jbuRCYXWuUqzzwzQMjiX5hBm/VUokhBHmvWH4of/G4r/uO27dpYbW4qMEJuW82fhZT+QcGwjNL5+7hZQ9xuId9ewrVvfS1ymQI+/vkv4eFd4+4+aWEiHLpuFd706ivQV3CEiwTohFZmpZCotywtKyf2QSECXPPxz2PP1Jxpdmo0MRIzGGN0WE7lrbCQggBf/uS7tUlrrOk7nMCTKch5EXMoCfHCt7xL5eIrX/YSrBstY3Z6BgN9BdUuKIRGo4Xdu8exa/dOvPB5F2KgXEahyHWzjIHxbzEXopjPolzIIlcqIUg6aDWXcN999yNXLiIT5pB1sVcmVxGoVF2qyn1QcbmpGezJUjIY9eCZMznB31z1uvToo47C6NCIBJ/PmW/0VS2PmXMn+jIq38uSIdOf1cEsGrvuwPCKYb2n1N8H1qLDIMekFDFyKBT7URwYQTbH2AG47ut/xI5FFnEIJpgtJZbA6DTPYM5CeTFWmAlk00Rwbzlp4bCDBvGH+7eDdLFcPsccVItJGJiVqDBu4Z1vfT0OWTmCX9z8R9x88+3YO79g1y8W0CYvkFS0NEGGcUsh362tJ6nxANBuyVfyXgnEEOPnfeTiOlqdWEAUOQkK1LKM6Gm1DIXMs9LJIkyWVTWWsyNRusJOAykrZtT0hG4kRSZMcP27r8Lw0ADyBa45sX76+ACFLE19TqhbtmAaPzW5TzB2QjdQLIPgVS5bRCZrha35+TndA91th7uMMQq5BdmsXJLnMcgCXv3Ov01POP4E9A/0qUzpmSI+L2XgoAjZ8ceIGQ8OjSDMpajNTCC751YsTe+WyeEN5ooFpAysuG2zBWRyZWRyJYT5MoqlfoRhFnGYw1VfuAW1CLpBCo4mnOaOJsyDebwHkidZQ0ijlrFhWGpkvuwCIZp9sktYcTKwhiRP4u+GS/B31A5FzTkSOwzdEsMna+VfQruMri11C7nGiNp1wdc0xdyE/EyRJDr2OX4RubAiXDhCYTZfVArMjED3w43SInBl+TtfqwJP3AFD5X++5rUYGBg03oDz8Uzr8rkMSrksysUssvmsyBSsMywsVeWCc7miaFf86L6hYQWM5CNQu8WFSN3n0fX2pNDdNPcfP/Cu9Oijj0bfQAVFLnpgCJonUdCP6I3coSI65rBipB/ZzhxytX2IOouo7duL6clxjK0cQ4YFCNa9aSZzXARWxXISfC5fRqFAn5TBTKeED33vbrFd6Q2I8qt2DeKelrrJF4fmn5NO0y28ESy4g1ms4AMGcYo0dsGW6E0mSNYJjD3kijq5vOruZAGrPiC+Gz8nNMzesWnQiUU8YZbD12nzOOSMfpkBmQiNciEeRXS8O2U+WQQutYxliex++NncuAS2WDEMgwSf+ofXYHhkRByCbM7cFO+3kM9K8KWC/Z4b7oEHHkA7jkX+LJcHuDgqjBl7LUB1adEwEJZkewTfi5P4+w2++rXr01WrV4vlwaqV1ziCFdqhpOrStBGhCjMkD2HjaFu8vGa9jrjdRNysYs9jD2JguB8ZmuACNZ10JQYreaRBCWE2L7+XLw0gn+tDjDZ+c/du/OC+mvBjZlOMSOlDpXUUvMyhOSWaRgrn0IP6sXXfEpKQ6R+lZygYo3wKRCogjXRsU2k8HTWZKYzWtR+M/0ZPyOditcuBWKxokc2ijeBJoEnarfi1Wg0XD9iG7AaOzl0pLuKzhgy+YrRbNbMQ3Ci0KjT9LuAM0wiffsdfYWCgT4hhzmt8wOAui3whlLknqBS12rjznrtQHuzH4OCQTDyYriZAo93R91p9SXEXuX9MSRhBJQ5V7Kad+n2A4Mc/+U5KQCOXz4hkwN3vH0j+nTCj427HaQfFxm5k2nPYsPEQRMSK63VE7Rr2Pf4QKgMVJEEWBW5ZMkizOSAoSvgQm4QBSQkD/YMIM+TlRPjkz7Zh20wTqk7QVwZMVag1zu+H1CQgK9Od4NzjNuC3D+xyTGBHLdZdG3tIbF2nkWTL2LMAMS1DYAJmakaBRdwkjCXSZZKmuAmuTE36uEyzYyZRGXRtugrHCtbN9RSaqIXc+Lwjlpup8ZaimZknN5/aLvgaMT76lpeif8BKtdzkSlkp+FwW+XwokkcumxEWQB4e01fB3glzfqDFmCXOY3qpij2zc5iYmRNPj7WCyZlFTE3PaN2EzjLnT0l3zyC48Vc/Tum3izkLSLxv5wsZFPDqeQoOQH3mUQwkS4iSNhb2PobDjzsJcZpFVF/Avom9QGkE+8IxzHcsKm52OjK7LIIwJ+bNczGYEkqzyRlfrKoQwyCKpVLyyK3yFWL16tWCbVetWiWK0Y7tE2i3UmTDMgiRkGxA16SFdSVaU2fXTOCid5pDWS9uD2/JaBIpdPpD+VwK1Qo6PjXzDFlqqzYV1yS0ErIIoO493WvyNY73T+toG8SII8IFGE+0m+b34wh92Rj/+IbLMDRQUVWQ68/r5sIApTwFTnOfU7DXaNZw74MPYcXQCmT7BjDZifGr/7odv/j5r7CwuKh7bjZaiq083Zv3q/RQjSP2DFIoupxb/vDrlB9AOpQ3W3yDSrREk/IFFLIhGgsz6M83sDQzjrSzhKWp3WB4Mrn6RDyydwaTM7NYmJ4WLNpqkDHCsqpl1wGjJUdOZIzAxgOqCYMaMlomJicRODIGF4qfS0TO4EvL9WnGy+VB9I0MYGx0NTYefgRWrdmARx7eiUZEDJ3mXi0SXcFzc7HkaigZwRZWDU1oKrSoGhd3N4AyBLo2x67hhvELpss6gEaBo29scBU2a6rgpjMLqTuReTerwcIIf8fYQTy4pIOV/UW84xUXm+ALRgRlbJPNBMrj89kcClTGDNCoV/HYvgmMHH0qrv+3b+Kmn/wUzaUakpibqS16FtNgGnLdpweedE1bG/8l2Pu2229OuSuIEgmWJFWnY61D9LnFfBHtZhXlPJDEVTSJ4i1MYms8jDu27sbM9CTI0m3WG8rzSXpQaZJa6FKIgCkSF5sgBzlkDeuCUTqmbhLyAai9xgX3xAziBTSBSptUuOH9RdIkslsYMwyvXIGD1q3H0aeciU6SwfT0IoKYKZsBJGCwaF5N2YMv+lBI0liCMNRALprzvd02JII0PW1cerFr6uBr+JV4eM9bFwnb/KhF/wbskC9HgXdY/ubnJh0cubYff/OXF6GvUjIGsKvO0UUJwMmhtTQAACAASURBVMnS7zM/A+qDa/GjO+/Ad7/4RSxOT6M6tyRhE71jzKB7UZxhULDhLz2Bp3sOX/0L/njbzSkrcTmmR2J0UvAdVYoYZbcaTRy0ZhSt9hLSxhyqrQQ/fGQntj7+BHbu2KViDh8iH2bRYTWo1VavF4kN9CX+i5pLIERmNKILMHap98Eyxu5GuVA+q+DfvQYyWOli4u5B+HTtVhv5QgnDB43h8GOPw4bNR2PX3mmkCWlGXATD9wn3d3NZ19JkqRU1uCPfq9cR/OFiOizBP4OYSq5nwN+HzwR8XYBK7zeUrbxzEdlQkCvXlqkc1+ysI1fiZRefp3o7LS7jWaGdxEyyxO/p5/OYHjgIn//eDbjlxz9WQN1qNlBfaqJea1hmwazF1ROM9r1MF19Wc2cRfX3k97felAouDPkhbDeyBgfGZwsLCzh43TraAbSjOqr1Or53z0N47MGHsG96EvW5qpkR+lpqRxoKsFhYnFckOjRozYsKimxFtC1ljrgBGEGLlNhCqVDosm60GZyvtZ1sixfzvU6jFMn3PCT3GO89E2aRKRVxzMkn4fjTnopHH92joE60aaVUbocpTTOzTpaQNmTbCBPmmy1OULDnzCbvn7IkV4GsIAV+jlhpG8HKjbpfFzjK1MsCpOqGMaoXsYEEr3j2GTjz6E2oVAhG5RWRM0dnUpvPBsrfp4fX4Gs//BF+8Z1v63lb1RqYWSxVG0g6ZlloKUzY5t+9lRKwxKyFn66mFXNxMvW33/m7VACNfEtGwdxAqYJGbQnDI/2Wr6YdAS3fvO123HHbXZidmUCtWrWOGknGkSmcxs7PzWgB+ojiuQVQlbOnGdIvKv9OCJMwr1AnSlDWzW7UUDHv5ykkBkl6TMtZXb+sqMxOQ/3DFQf7cNqZT8bw6i0Yn6wJE0ji5cWhn+X1fDCXOFPPq1PjPa/fkD7g4tMOw3Aphxt++wCa7Eejm0jNaoWsx9HfuoYNWgLhDS4IzKYBWu2aijtJRFcX4W1XXIzD1q1EX39ZcY1RpcgoNnpVe916fOM3v8F3P/tZ1BaqhgoyaK7VQeNET8brdxtCVX1ZFrA2rCd8sMdOWY6hecG2HQ+nytPNXuDxJ57A0YcfoXowIUxT1A4e2LMLN/z2Fuza+oTo0Z1WJLSNC5QLrSDDYExtU0xX2EjhCjVSBEGvy3mPj4yJhjEIpPb5WrUE3omF5JnGEZQx7bTXE41yLdRsfHAVLW/GTUUNDczm81ixcgVOOvNszNbLruHTbyrfsGnBIz/TbzSfx1twB1TyKT74mmcp335g6y58/IbfWZSeWPA0UExx9tGbMTg0ALJvdkzXcPeje9FJXJFILeANtJsNVQJzYYLrXvd8rBoZRH9f2bh0LgilArI28rXHHsO3P3s9gnobs9UF631okyzJFJNt07auXmFo0cTjd7QuAW8eCEnNTbJ2IcewbeuDMn584F27t+PILWSjLGtbSsJDp4Mv/e5W3PmnP2FpsYrFuVlpL1E9+TYX6PhArN1q6Ca5YqwZq0ecrcmwuEFsWxclCxGLY3HLuNhWwrTAiF/LdW+XirkHUBqnaot1wfhWKh9t+9hAGiQwpIC1h23E5iPOxkw1Ul4fKge21IqWjXi/zGVkm4zBqQI0JHjds0/BiUdsEMBF3ttbPvNTcQUOO2gIVz7/PAz0FY1k4hDHWr2O93zlF3hk15Q2ra4dR4rASW8uFXO47lUXqWuGtHFDLRkQk4oVYm5sNf7hfe/B1ONPoF5toLG4hEg0MWtKZdm6G++4YpoXfJeswt/njJwiM2+9WsaDePSRe9K5+XmsX7MGCCx/FnTioMqApcMgwAd+8GPsfvwJzM3MoN2oi03q4dzeHnANFiCCRi3nYjKQ4W5nBymBA0er9bvS/5uoIXljZMowyzDs3ARP7fZt5f6BfdVQ+DbNGbn0Dnvw1/RWhdaHPpQo0Nia1TjhjAswOWtAjG16mnWn9Ywj4tRtVFcoCgNc9+Iz0NdP1GxYz/APn/gOLnv2Kdi4akiVSNKoSZfig6saFkW48iNfxu6ZljYPg150Wog7LP7EKJWL+H8vvxCrVq2Uj1ddnSRMRuO5DH40OYWvffjDyKUhlhZrmJ+ZU3Acta0TNqZ/d5aOz6D18B7Qde/qn+x/cJCzBG/BAIId2+53Pt7Ff0w7HFNUQUkSoBp38I7PfwFRvan8ul23smTiWpx1QZcoehCIQmfpVakSc2kGLs6HEV4VE0abzOWdaqNqSPs8iMRqYLPe7sKdPupXHaDXnCk1dJvK5azd6N3FCXzkTDY0GHRwAOdc9Jd4YjvhYm4qq6AJ+KHQ9R/dHwXPew9w7UvPRH9lQIUUami7k8itsXTKz+qrlJV6Gb0a4iy88rp/xXStZe1EHSvwsGWZ3/vKeVz3hhdibGRIVVG5L7c+gysPwT/dehN+8JnP6P6qMwtoLbHjJ2PDHshWcmml4hkH0BizyBWaHALLTKZbZHOMJHEHd+14kFVHV6PmbjI/4YVPwd83PYWPff5fZY7n5+ZkchTYREZGoKaxYCKBqJKX0YL5luGUwxKSjh7MdhzfZ2M7WEnTZ6n6xc+3yNkHcHFkkasEaVmquXBXePGbRDEhNcBPvnCsV6/9phXcIHI4GFq1CqefdwG2b20gn83gnGMPkRn/7n/dxZKhLayvwgXAu192FsrFigRPIVHgCgLZxMh6OmOOuC0XwveOT8/gTf/8E3EXhAa2WNjpICVyl3YwUAxx7etfqALNgOfOuecc2nQMPvbv38RP/vXLlAZm9hHgksd1LsjRz3rmAsiUZ4ysaWtlcDV9vA98icR2K5+7dz6QygcIraLf7MV4yBMP8YddO3D9176h/LK2uIimIw9GrUj1cC6l0DUKm4tSKNrCEaZkBCn/Sf5XR68hN73XHHOz1KqkdrnUR8iYE7KCq9AKHMs7Qu/3voubVQ/sQRS3v2je/UQMml5x113vO987vGoYz3nui5GPs3jSYSsxumIIP7nlQfz89ifkl3NphNEVfQg6EV777FPEFciRaCJuQkEAlPAOdSDF6sSp1uoWOacpds/U8Jnv/Qbjc0TW2GjSRqfFGT8RBgvAu15Hwa/A0EC/TcfgtqcVXHsoXnf1mzG5fatKzlN7JtHh3IGOwcm+zNoVLhXJTwhxZFDx7DXQwp7ZK7JiCf6egtcOcRUkXwZ1ayfB/+qhB/HV730fGbJLG03l96VyWRE/YUMPanAgAS9M02XRsHWMdtqRmjFs8gQrgMbn4xdNF+MC+kDW232TJFXarsF766mC9RAlfflYZt5tPrZNd+MIEhBcOsWF55qqGOKsAu3Ohk3r8fn3XgeNYBChsw0aeQFMCjzbyDgcgDV1wxCdFWIwB7aBM8hNMTXJoQVVDV/Khnm0GzU8MVnFxFwTESNql3qxBFUuhDjs4DH10omHILIlkC2vwOLAClzygov07/pCFZ1mB20Ol2p7opdLZl1G42XmgzplG07wHAph7CbPHbQAO9i9/T4J3hcTlArqhYa6Maj/z4fux5e/+31ZBX6xyCL+eQx1frL/2uBJE1CxaItLTp5cAtOwTgdlNxjIm+dljSWJoGpUoR6Dw3TQz74hgdP8mQV9rO759mb/wIpJnCWggBmWW3rJoIj0Lr4vRSFfthjFggYce8KR+Ke3/r3VFBw6YN9tuJBCHocRMCAkoqaRCMp1m/pMVtHsy+BpFmvkXlzM0VvA6xZKHIrm75vSKY1swV21GVz5ssvlPmenpsCCe6tJi2kVSJE/3CaSiXdarfV0d2FO2PrzFN84S2DE0RDBrm33plbNMTOrFwtbtxunlm+dmsK7r79eo7zYfz49Pa0LksMWkbNOPyZcm5W1SIKXRlOQbvAAr1UgEcL5TW9R+JnUdGo+f2Z0T7fAtmUjL/ohRRYjdWnTLK0q1bL7VZroNibzYFW6OP6M07ESG8ZEU88qPI2z0kg+tWvHPvPME/G+173WWQubKME14OcRMeyicc6dMDKXSVfjlJl2GzbkNjvDFlcA8trWGzQ7jnVXG7VJMgWs2nQyfrvrYVzzt29WlD89OUX+F9qiSpu785u7m7Y5KrndiOvqcZiAXusKNZIZ14qbYPsTfzJT74TufYU3lwRdluIYV33sY9izaw9WjKyQORNAE2bEvo3qNk7MI2Z5ES4ziv797zTPxhcvyHdj2ZIkxowVaRrNpjB3sk206TizjTmcQ798dcsTNdQz59I3+XE/G8fh1EqpOJPGaYcWSUkE0zZHRhC1i6VMoNzfhysuex4uOpkNJS6ecOsiDXVAUrfjV1mLzQEy6Hg59LTgys3qcTvcv6Z7bTapOqSQm0XBbHkEJ552IX744O342LXv0maan5xGu2Fz+biBvUWWn3cWdVmbrTZgf7PmjO5XYAJn3CNTv/WxO/aL5gwNNRaMNgHBlzCDN33ww9ixcyf6Kn1inwqQcflqa8nmyfmgg2wer/FKP8IQfUxZAvpO02JW/riYziIKtrWCg2kaF0OQqcMCLE0xbdKmFI3bNpt2tcP0lwNEe61gaPc3EiK50RgzeOugZgfahlwGI6uGcd0rL8eqsgE3VoFzNWz304EIoyeKShP3Z2Toc+lQ7AeLDZQ1+c3gt0vQUUo2sPpobDzyqfjmrb/CZz/0QY1dmZ+YRrvZURWOFsBruy7hNJ2/M/KKZWTmEi2GkrZrjay+z79L45949Pb9BO/RnS7+y3AmCXHVJz+FHTt2mUA5k6bRQKlYUdNhxFzbTYOU5udC5IJQ06fYj81FZMrDpkBGwuz0ILmQr1XFS926ie1q23eiIkuPxKaxFE/+TNQsg2xlrknRJj6uoYVu0uMBdCNR8Xt64nxFjUGnf5+lPMARJxyGa156ETLUSEfA6DXRvaQLm79nFT1vgnutp35nXG5Xo3d7wAWtXY/sovK1R12MFasPwse/+Gn88IeMqYD5ySkkkbVs+U3vYyMGsvwitd1vCG/apRgug/EKwPsVY5iA138neAV33RZhUpECXPu5f8EjW7dK4H0D/TKRHkWrL9ZMu5wPCYwnpfStVMx3aT/lkk2x5AJzwyzn2AGWFmwciEG1ROIsImcngP8d8XTjsftq1HKRpGsJnDb5a+vhGR73jEZl4YJfrTpHlbQVRKnuEDeRLZbxgueci+c96ThZGwWBPdMovUXxwv4/v7Ms263ULTd2UOhe8N4qHHfmy9AulvDcv3yumjKrC1UsTs+ps9lrhH8uWVjH2OFoWD+mrbsONPU9FrHL//f4x4GC38+H6Kksgvz6D3+AX91+J/ZNTmPlihER9Kkt1NzZqTkJQ0T+lEOEbKJUg+PHOEdOXaaWRlhbVluRsebcudIqW6v4ZRUxC9i8pgkAcUQNPxOPVoAFE2M1G2BB089Ie7nO76ZfMo5wjFsjaFre6ytwvjpHAbA0zf759771FRjmbDqW5vTN3tNl3hxQl/ea7u/Zm3OBNu4f9gzuOiqp0nbbv/m8p5zzKuyLY1x8yYVI2x3DTJbaypq8Jve6VFpemfWsZVPe11NxVJ4mXOuCX+HzPRhG8PgjtxnE63DcA4M7H93f/8QT+MfPfRb7xqeENDHlZb5OwU5PzMgf2pgOju0IdeP0nTRRjNR9p6lpl6dsW+uxiBcy81bb94vnYwbTKm/q2aded6NOjTxiqZkPZJbnxskMujSG16LwhEp2HL5AUEn4dyR3w0IKcfNGp4VDDzsc1778Ik0IEYfAWQxtHIcNeJN7oHk3VpFx7Lw2+2zGx1tiHYnla7uCKdZJT389djTn8ILnPxedelvZUmOxDgJlPiXrjb+84PkZJlRvqYmeWvpLOSnO6Y5pdXHC/yR4v2M9hZQ6e8Xbr8bknnGR+VeMjarkyKDFplVbfkkiBunCNKNcNM1+4ZQot9i8GU8j5mf48aX8O6vaxBMOFLwewOHntPISpjRcW9YshWRqpeVljTfT6tunVWdz2YgXGrEDVhKXLUyKKG4jzGVw8bPOxAufdCJsAJ4Fe70MnD8TuIJIY+76Qpeyu57ah4tcZOks4+GfmXEkOOWcV2M8buOSSy9Wl+zE7n2qzJHZpC9qdU8rOF2WBW6ub8CGDysG8jELKdi9BTFqvnoi/2/Buy2QBnjde9+L6YlJ1BttteV2Qkb35JSRTsVBBqOYn19AqZRHu97UBAcxWVUAsRiAi0Vs3LTBEEMztQQnyJV3wEi3b8+CPbJNJHAVAARDIAxp1m3OjUYnyGotR/8+4PK+jhrPh+a24ZeqZq6+73237iVuS9Yjq0bxrle+EKP9JBwaC8i7pgNNe9ctuUaGLqPVW9NurOAYPb0ECsZHYQnHn3s5HlgYx2svv1xDlnZyXm2DzRd+MzlAxltnx67pFmnYs+i4CrbZrWdgOZay6p/WsVfwvQHRssZ7wQPXXP85PPjQw4hbxqAt9pUM3NCM+hhjK1eiVquqVZjATnNpSa1V9SUifSZ07ThXRyf6Z40PXviU3XIwxfuhpis3pbhcNUlpXcrJkHy9VarYR+bUwpENliNtmVJqhhtQLCF6mJobxY0oMbCIrNsYaSZALk1wxMlH4e2XPBMJ81ovfJ/f76fJPtbowQDE0LGClFHUjPcvSmRP+sshxtlwJU4454XYWp3Ei1/0fAl+z9YdaNVZOXRkDnLundnWWtBqGBnfSCeCqx3IJUw+g5C9DS7rkOvz6R0F37sjvL/v9a/ezPzyjtvxuS9/w7LTJEFf/6BAEuaM1Wodo2yhyqZi3HYaTTSX6IsLaDc5A4+948s0oS7o4Lhv9PMH+kx7Tw/BkprB4TBuSoVnk0p7e3y8sUwcO8VtBy2My2098GHgi6F/QtkI7XYJl4mme3AcyWUXnY3zTtwiq+ILJb1BXG+6p2v2cvV6wDF/T5aWmpn3eX2mshknPekCPLQ4gZc+7xIRR/bt2IW0nWoEqwJAFyAIqnYceW0gujONRjGkUabd+3xNyzAOo0y8h+T/O8FrZ/QM9vc3vGtiGld/7GNokM+dJOgfHNIN5Esl1JaaSvM42WpmchqDlT40qkuW57rOFAqeXz618IQLQp0+mjeTq080Abvac7cq5SY+9lokWROhaMZt90CP37wezu1uZpfOMeL2kbpZF2sX0+9oxrKhZr2vPmQjPvjaS01QnAbta/zO5HqLpXtydGsfzPXGAQdaUWsGseccXXcqNh5+Kn6382G84YorpNn7du1G2OHQZXYYWVTuhejxerOgoWb6UuNVYXCC1wAoR34xsGx5uNKf5fFeyH8meAVQKV7+9negsdRUF2uhVHInOXCEZoyBgSHBrgnZpBwQmMliaX5hGRNwJUW2QcvvyiVTUNY9Y4vEvWScd+1mZ+L9QtJskg7uLbsXJr/3gjzK9Z2Aeydg9UKdGhQgrGB5uD81nuwWfn6x5Kp7UQcnnnQs3vr8pyFhAEuouMubN+vXjd499O2kvHzfznKpIdQFgT7RC2Ks3fxUrDvkWPzbHf+J9//91UJMJ/ZMIMP5/4504S1ibwbmTbfGonhwxroQDFdx5p9TM2RlnaX5M8F7s3Wg4FVxSoFXvfNd6h1nixRBbqZz9DPs1SItScWWZlssXVbXmrVal51DhZF2OJ/LefDC792pE/74Ea6Zh0u94HtNqyyGI17sf2iApYP+iw0XfA4fsXdNsouC2XBh4IqnYBlvgMEqNy3rBmq7Zg09l8ObLr8Epx++1t7j8IflWMG1TrvY04J5l8FrQ7syc7cBw0f+/FuMw4+/GANjB+Mbt9yIT77rOmVDCzML6gTWejm+nA9Yl92FabH66RwobHgJXSLHprtBEY65a4qSLAd3+5khsTmWmyGW/5bic1//Fm659143FaMtrlkmzxw5oxnsNJXkp7MnnKldwBMZ2k2n4baQojVp5y0f9GP9ZHxI16Xrkbb/5lAkE6blrUyXvNb3+lrNv3flym6q5iZlmbl0ubnKrsuRtoKv0NURHKDE/J7CXrlyJT781iuQURVwmW/vJ2n6dTrQvNt9LWMBFoAsX4P0miNPuRylgWF89LtfxLev/4Lq8NXZqsUVztR3i1yyGm5su+M19Lo1tZ7J3xPSJtBlkT3nBHD+kCJ+H9X3Ct7vpt6gjxuVulptpXjLe9+thgIb/l9ANh9qxh13HevgnAUbtRqqH7Ma3G6Qg+5GjKo/3Z3M4HYhP88iV5q1XuybUzCXaWD+HjXT1VGfeMxIt1DjxqHZ/RsB06dy0pSeYr9lGGZ+fQrpFZQuzUWH1nDBOCWw4connHo8rnnxhSb2nqi+F9b97/L7XsFrI/QIngcRHfekVyLfN4D3f+Oz+P6XvoL6YhW1+bqUwbtf8fnUEk7XbVmO/8+ex9rSLO21vn/OxPGvMSjc4RqPPfzH/blWzkQtw3+2BqoMyc8neOW170Lc7KDW4I0lqPT1axIGT4KgeV+YnUfSbttkKJ2SEGkBPZZPky7SBf/ncHdNvhaH3wSvmXZuSrSgzq4sXErYZdosQ578DAIcytVpDTgqNJsTx603S/Edtt2mDBdc+nEhSiFdKZYLau3ONpuWNunNf/UiPO24TeikjAF8N+z+Gu03wn4Rv13VxTLELXyXTQfHnv1aZEtFvPOTH8BPv3ODMqOleTaX2nxc+3IVU5uNLlqV/u4yCV+UUXOGS/2ISfrfi1vAYhrP1fnfBN/VMHd+mvdb//CJT2DP1JR8PRejUCxr5CajevLp9uzcI+5Kq9HQOTcqtDgN87uXBRdj4jpSINMxtmARPOkhG0gj3YSpZY1f5ot30yEH3XrBy5wTruQGcaNWbJHoIhxh07mTLnjj0tRumCDNdBOtuufoNTE4Oop/uuYNqGTMTRyYvvln7NX85Y3gy7Q9pj6NcNLT/kYW6lNf+wL+5bOfQaNWQ7tu8/a94AlWeRTS8jKL6Ak7+9TWc+q8sBOljL5knopnL9i8V/B+d/aakO5iO43nv+fabbzlPe/TpEvWszmtqTzQJ23rHxjA3p27kXYiDdRv1xvIaEdyopnV5mlNBJa4yF34ucCpZbMuLXcVbvu558uf+uBOiuLDWqmV48eJ6pjfZ27PQoUGASjiNW2zcwNcW3NPV6tcjidhmC7p9dZfZ1VCC/5iHH/8Ubju5RcjzbigqtsHv0xqOdDk27+XBU/6uTZJ3MbJ578RnUwGV13zd7j5t7/B4gzZzHbGzeWXno+DRytYu3Ytthx+sjSf+AnHovArk7cDDLiOkZo3OqJ38/iS6mIVu3btxPjUtNZgdMWIxrsHjz5065+ZehmVnsHCvaaeP9Mkv+Kad0h41PhOJ0D/8KBQqpGRFRjfvU+CZ3GmVeOZZ4ZW+QYGCp5+U8CJS1XsnDTDnHvNI9l/vRG9F7/OaaPA09jGnrkqneBLsW6tVu+jenseG0fSi5z5wMtyca/BDvVzgRWbQvjF2IQ+ts5zdAb68YaXXIInH7vR4fcuqncuwt9nr8n/7wTvLdqJ571eJK7LX/ty7N69ExM7d+tcnA/+w1+jsTSuruX+8iBOOvlctOheOA3bATtqi3R1CmIZhgoukzbM+jlfryyXnTQHCt5H0YEt3oEab4fsxPi7D38M+2bm1KPNHJzjVGTys1nMzM6onMlyIjWe5XCBIq4Y4mqpsgJ21lsGhaLNZ9UZKgfUwL22q+/cgSbGqzNwg0ebLAekPZOhHWDRfWgXqBhGYOe8+SKP105P+jBugINhXVRurdNWziV5k6dPXn/t6zRShfN57b7deXvupn1N35t/g2z5xSPI3FSNNMAZF1yJJhJc8BcXolpbxPzEFJ739NNw7ilHKzvZu3cv2u0ETzvvL2y0W4YFsZY1RSqEtuYILU8P/iHShYO4FfASgeD3/03w+2m94FPpu4KSG/90L7763e+KK+fPNB0cGsYS83Z+eMeIGA1W55x5p6n3QZa5E+ukocayuyTmQAP23HVbq5fNpu+y8ILndcjtY0DpgzSZbwEX1o/HyFb5rzv7zaXConJzg7ISyE3D9/cya/wm8FG+ByIMjLHNEDV5wEEbp55wNN7xmud13ZQ/dsz34nvBd69Jp6TYhtVIA384NvbsZ70ZDXRw3nOfqfR3bnwSV73kAjVu0Idzrs2WLUfisCNONndDy8Jj3kQbk7S1bgKyZLKZvtHF+U3hu3pdJuAF3+vfe4M6X8mSeXQRqRinaYqXvfOdVp1rW55bKQ8Y9ZcTSjkgoVnXMIBC1qL9ZsOgXp9XMxU08gT71SC3wQKy9c7v3z3bTWV08C6DthBhjhg1I1gKuqPhTdQ4agg/Y+P6Q/T7J3bv0nc+QYFM4E4kgKRUKVvzB+/XUbcs6nbDC103Tm8qJmBJPspGnw8OD+Dav30lDls5pJGsjPIP9O0y94Ejk9AySPDGG6DP56HHZz3z9SCP6annPRWduIVocQEvOf9EFDJZNHiKRpzg0r94EZJMCXc99ATufPBe3PfEds0XaqlBdRlml3vTBDHWsK313GIcp/H8+ZEH/7AfEaPrTx2I0xW88416KLczrv70P2Pv7nHU1QiRiK9e4kmPBGg4cG9xHs1qTa1XFHK9VlVaVGBHiqNQ+SmWjI2I+ok73jMU2PPIfV+ZzFo2QKWYRV9fCUdsWounPOVMnHXqUZpLx5YvBWX8X8+YEl7zZzffieu//WNN6uJCsAlSvt2Z5WV83R5wWfPN9xuubwJM3TGqTBU3btmCj7z5cimdhhj3VO+6m8ALvksv94pEjU9x1oWvx2IS4YKLL8D87BQKnQinbFyFUilEK83h4aklVJsctJxBJ43sEAWlecQ+HATuXZvj01tKu4xzCDQLHHT7yAMH5PE96JaChG7o5wbEdcsnwHd++TP85Le/F1onDh1CTa6iH6HpnJ2e0lwZGh+mEJx/y9/zNTTBbe1U46bSzDdaNVWjSOvK02wHGR1Pyu5RNimefczBuOaNL0auWEa22G8bZL9wX2Fo128vM1qXq3V8psvecDWaHfo6etrlnOrLdQAAIABJREFUUyVoxs0aeaH7s++6oY6GBSt9SvxxqHRRCS574bPwgrNP0LHf+wvebWSX71NYxuJxfYc8H69TwbnPfAlum9qFv3rBJToAapAzfJMY2VUrdVgz14vsZimmKw9zvT1NWemby90Va4Dzh/O2Pjxjhz/buA7boA/ff+v+ZdmeAwB6BW94ke0C3TiAxyfGcd2nPt2tvtHskHdXLvcp6FuqLii4o49XvskTpjsWCFr0buNLKBa6DPo6FWs6ETauGcKpRx+FVZkW+ioZTcV68gXnoNTXr5mwYaGvSy1aFsufC94s2DK/3FLDBB/90vdxy+13q7ikESqOmOhNvQWLPqOwdNQqeNZBq0O1dW073rRvbAj/es2bNQv4QMHrda4L2QteZVKXiTQ6/XjqBZdhW20ef/mi56BVb2LLyjE8OrFP1TVyA3RapROumLLi6RlY1T1hROtMZI4HkCyPPekOqGQzhevuleC1XC5a9qdGdjnc3VV1gu+ZlUYm2LWf/5waLSi4Rt3OSunvH5QF0OTLZktNlS7YVGBF/63+OlKtoibWjo1gKBfgyU86Fcds2YSoVdcD7dqxC7XxvTa8MJvBEccfiU2bNyIln8zNxe2mTeLjOwxeW9ohjTpE0U2B8IvvovrPff9G/Ow3v9dG8C7OZgAZ1cprfm/MY0pj7dR+8BCZxwxKTzzpaFz7+svUb2iwrxVgzD0ai4auwCqCdm6u4vvsKpz5lOdgMm7iac94Cvt8sFSr2rkBpYIILzygkCCZGkRczq5Yh/UIxT3ugV3NPpfJWYDrqWou9uJhN9qu/5PgvU9d1qYe8KHH/33qhhtw59332KSodltBUqWfB+GWMD0xhYQDfHnkB4mYmVCb45gth+JVL70Mmw9ejdt+eyNKGaAl2lVq57W1Wf1b0oOPrBhFpZDF/Ow8CuUsTjnhKE3PDDlwWX2qjnPnTpdga7NFuAFml+rYPTGDJ3btwa6du/H4jr1a/MgJNYMQe+d4+JHx69XoofEtHk9YVohebIGLHDUtoGUBhCAWZVmq5PHuv/1rbDhoTFC1xQn+9Gsz+ewgVgbhLAp/Vxk7AkcfdxYerc7geZdchAyVqNUSNsIDhIsDA8gXy1izdr1AnJGVI1ixYrR7uBKHJmkABYmjUUcnWEQ80pTdSY4E09DcnQABEUhO5/CC7+5q59QP6JZ2Zn65YGBPFePGu+7B17//fXWnkBUqfD6bU8co/dLsvgkcdtBKXPv2v0eZGscFcQ2PRPTuuPVmhARIskTAlufMeoKCtKbTckeXt3Dc8UcjIjBT6dO8WBFn2XHSbOBHN96E2+5/RFOz5xc4vIEjWW0fdNpskDDNZuuxPUkWHNPKgMdAneWDE4Q0us1ghxQ57pqbasXOVf7dmK02pqUV1TE0PICvvu9q66qVK3DBoOPiJW76tbFmLfXadPRTMbZ6C+6c3o1XvPRFiBZr0vCxdWtw/AnH45o3vQOtbAGLSRNtXoeHKDLOIOdQQE5TgheLiC4kxz5CK+ho1Bt7DgXKaWqwgu//UfDLhYHl+vay1V8G++ZadXz4X76IfRMz6g8XQ4XDQfI20+bT11yDdSvYnWrvtvzdH/CT4t67b0UhZKQKneaktIqATj4vTIAFHg76L+RCVPpL2LD5YLTSAm689R48uGsvanEbDRI7NayYAmCDpAmEEueu9314nnZERJGLwaEMPJ2Kx4ISG9XwX1f77hZ12AnLmX3uqBYej8b3b39sG2rzi7bAAa/VUimUtfvXvfQv8Mwnn2LxkGsIUUbAymPkOABdMmmKE858Psr9Y3ikMY0rXnwZpsbHsXHzFnzn+i9isDyAxRCYojYrM2B3bIp21EQh5LFsAZpRE40kknvlBGveY7vdtJZwztbNZTVFVKd1c6Q6Q46H7vvDfsGdL10uI077C16+xEnRV6T/8StfxgMPPGoYfKOpAf2CU8MQ737Da3DcxoN79oyVZ81iJLj/3tt12jE5Y9wbGvTnqE9qiswVcffObdg6OYcmkS4e40VtijqIOHyJ6ZXNf3CsXetatSKFaWmxwDHqqYQnxorr+KG14EZbaiyKPqaqHUu+hbyOXtFcHfbQpQl02CCPAUkTneTU3z+EQqmgMXC8xvzUAh668x489tBD6Bvsx1fe93eu/85Gu+hxCbeIim7m3yqgIU4+66XIlSq4c3o7XvXyy9FXqOCmG36CTjaDe2tTmFiYwkJ1CUnU1LNVin06P2igUtZz54KcKQAPbK5VUa0t6dACYhWe/MKAUCdq8339Ayb4/YKXIOmJWLVnl928+6k3g+IDfOTrX8KOfVNYYhM/o/OGjfwuVUpIW21886PvWw4endYbVSrFI/ffaV2jYYDhwiCWwggP7d6N+3ftA6e9WD5uQ5DIfy+VCAtnNJmKJj5fsgHLImW6IUd8vU6iEiOVymzRr6ZDaDqIjUenQDz/j/dLS6Hed3fsyMLCnH6m1WAA55s0+R4e1yZ2TmQmv6/cZ0WifF6t2SPFPE47chPWFAjqOJaP8n8P2bq9n6Z40jlXIFcawKONaVx26aX49fd+gioifPeeW7Bv9x4020ZWpZvUHB1X32DbOT9P5wNx+geha83+56idpmYOCH3V8CgrK9OtqavIC753Vy6nKlbrPfBrP1oRgEen9uKr3/sBduzYY5F1DC1UpVREI47w7fdfi4JGoi9/+c979IE/ycT+6qGHMKHZM/TpHbFMleY5/0QjQ65dsdBnlOwMO3nKBssqYjWfyvr7gU0P2YxtDsKzur6iXYNzaX2kyc70coPZWbBkFBV0BIv8uwNFOFmDMDXblnTEaLVuWLhmJLlBDBqz2gKZBfTJlXweh60exbFrVqLAw/6kOZbOMoA97vRLMTK2FvfM7MSHrrsO1/3j+/GlX/0YtWZDKHwjsvI3mU1SRTe7lm3q/L2OSHcDE2z2OQcgG3pJ39/f168z6Q2Asna2ZcH7kqXPT33x/8+jvP1KpMKtA+CaT38Ke3btpeHRTbTqdRtRlglx1MEH4QNXXWlND1phnuGQw9bJCXzlxp+iqeF/Hevf1rFlxqnTgmesLas6vyDghydcqFhCwZfLNoudqKF65G2gAdeVAmabcRe75sGDPNpEwjZrQ76g+eHlXj3l+SFkJvmz74ilC+Ln8h54f7wWByl3hxvFdlIlf6fqFzLa/DwpQlF8QgIErVAWmw8aw6lrV2GIz1EM0LfqRJxw8tn4rx33497f3or8oavQzmawZ99eo7g166jyUEhWNDXg0CZue1STsuY9ERX1ZW9aAI6Cp1vSc/oBlAzAKfyuqfeIneOieTLhfrNJnML65gCvv2EnxTv/9bOYX1jA7CzPRcloECJbq3gWXV9fP77y3ncgdLXoWpDBh7/2VdQ4NiUb6oiQYp6dtBS0+T0yham97FtX0NbuoJ9DgrKmvS3Oi1NbtO1gTXB2x4F6mhf9Hx9SftpNxTTiAidulG0sunwfq3vmq42Ry7P1LD6Ym511J1waLz+roo65EgqFFoAADg/3NdNvk78ZTXOEO6d1G1hlYA/LKszzmYszRz9qzTqcccTxeMa5z8Efdj+EY9cdii/9/scKPHfuG5eb4eeIE9COxGWk4EV2FW3dOo/ov2klaUH4HDq/p5BDP1FOziEin4BuK3KnZfYKXubCC77Ht/cGdDJSPTVzL/x//+1NuPnuO7F376QO/SHPnmANtY+jxZ9x+ql4yYXn4+a778FP7r5LTY8WgNnid32tZ+BqegPPb8/qYfg1Nz+HFStW6Pw5G49mw5asvNvRYpG5qwEA7nwZ1eXdDHrz3bQgoYY38ShuGzHuJli6oNAPHKBPlabHHeXMS9Vqd3gSNwCFwvIsn4MFG97nAlubq1U7FoSVNzfixRNMbWRMoHHnNKp8xv7KIC48/VyklTwuOP0sfPOOG/HE9m1CKcW2nZ1HvVF3/YghWi2jsrE3kW5LVDNOJGvUVSuxCdaWnjZ9+uh6+voqA0a+3E/wPbTh/yuo289fU1vCEFd/4iNYWKhpGjUVkBOyeAulgQEcvPFgXHjaSfjp7XeI8EfByyfnKNiiLkchtohLZ0JVzTS/3REofSbAYI+WwOY4WRrlhwaYZtu5NLxml11K4Wv+KwVIjbWAVZ29jrTou2jNh7puWneqhI/CuxbB8d1keplpMDPgKRsayWra1p3ooTMAjEfohyiYh7comxuBFUaCUayzX/6Cv8SetIaZ+TnxG7Zu3ar8XE0scYLq3LxNv2KwFxEws1OuRGyRGyNPYXkursrD6mewdjVuECrGsuD/jDpki9OFcntKH12hH3CI3ds/+0k0GhGmpucVPTZqNtRIc2Q3HaJhwjR/vDGdZknBMmcv8EhR81MUCjXMTmCsKHCisBgQSUhu5IiaHbN8COIFLX2n2aW7oK/lG1ivl58OQplgnbjhzJ4f70n3wSDJV+Z4v0pFdUJH3tqomVE4lyKAhNTuXM4CLlLIXYaijdeBzDADRDJ2+Dn8PSNsfbabK8DTJ7wbsvGwsY5Uo5AGDlqJJ537FGzfuk2pGcvNtCzjeyeQNFpoVGvabETl+Kw8a0mhk07T4vApy9U968jGwtrBg1AtweXxCmj8cVVdyrCDGLuTMRzdYZmdIF/TuzE+8fWvYNvEBKrVprB7Tmmy82dC9K8YxvCYnaXOPFrRdKXs8GRrCOC1Cjx1SVagoKofTaHamkJju1aKRQmRm4BmmMGUmgl0Ph5HtFD4oSJdHlIoQTnrQAvgF0QWhgER74dkkBxHtFkwyCyDGtls8v1sTc7oc9hDoPo5aeWlopWRHW9QAx8IALmxo1xs/seBDxQar6l5QI48yvunm2H0L1eSy8taaAN0Yqw6ZB2m5+ew9uB1WGpaUBrX21iam0dSb2tsvHx+HOu93IA2JdQsmT/3zub4s0GEOAnn+TuuwYP3/j61xTlghu2BPt6pucesZQ16ulb473sefwxf/vH31DI9OTGHQr6o1Ee48+AAVh98sB1Nmg3VDcoGDGq0zLNj4vB1FDoXRvmyNCpAlnVoQqSOOSvf6o48UWzSPQrMDiCgNjJgZDWQfycSSC1TuYSU8EpFAxa0UI4M4vv7/WYmMEQLQjfB82vM1Gd1xKgd48n4wE6I4t8NCzALofiGpedm0xpINIPVrAFfTyvjLSqxczWNJrZxma61kxiHHnOEaF08XbJEhm0mr3N2o0ZLhwtatZAwuKdpG+1a13Xt0lZwshGwJjNXabz/7t9Zde4AjfcVq16N9ibeC/9AwXOo39s+8SE0mxEWF8m1ywp21TSMXBajBx2E0dFRTM1OyXxT+NTu4eFhV+hIBXuWSzbtsdJX0QBFLThLkO7kDC8gj35ZfMB0y7c5G8uFAxm8hov5oxOiLGswHpoFexFTsB5yKV/L+6vWaoKhFQsw/qDbopVgOhVzWBOjbaNPSQDq+TOmLgtWtAIUsqhSOm/Oavn6HV2PQxap8Uz1CELxWjOTU+gbHtIZczT9tbkFJM0I84uLQv40ccMxj72LcmLt1hv8rF/rVvIbgefsulnB9931X5pzR43vFayn/nZ/2fPDMqazHAf4zfC2f/4Y6jXOrKPW0RTxBApCjQkqgwMYW7VSJowaNzDQj3KlpIhVJyGHduKjR/WGhgal+eaKLKf2zQKeI0cky1MmqWl2HLdZCk260vwkoiuWHtq1fHRv8YGVNN0UrU6Mpbrl8JoL70AeDwFzc/HavE9/eII0iqddOl9NzNxo2NY7wOfz2D/vheZd13Puocv3Szgh0/n+OMYSz5yhu8uRjt5Gp2F8Bs3+cz32XHc9k6/xusppnLBAQ9DGjZ3pys8Njrr3Tzd3Bd+bpv1fgveVp672uw/+xNe/im3je9FuJViYZ4pT1BgzPiyPHx0ZW4EWz1UNM+Kr0ReroNOJugQNLqhP88zk53XiIjeLD4i48GZuE12b16FGWquz5eMKLFmo0Gxao3Ornq2UyooXFA4hT9LH5LPJSyfzRXPeeVaeTZ82KNfq3/LVDgWTmddxIxaUskjDz5J7IP2cfATm7AUSSjtyORQmT6xmcEaloPnX3D926XJjRG1Zvdm5eRFccwULUvkZjG98u7lMfc9Erl4l9WCZZh264FOm3R2lEtx3501/jsk6qEGvO+Dsdf27p8nwwL/fct+f8L1f/grNRlvCTHQSFGfR1+RnVq5eheHhEdGFS5Ui+ocGFeRRmymkpXpdUCwBlmqVg48NauTf+BrCrjqpmUOVNJ3aOPq95t80gEMMbCqXMSoM6vRQrVqdecx52w4r5rU85GuZQYQGMXIaAyJ7boQqwR9r6ba5fPzZ+2w+o9c+Rur8PWuVokS56ZtKK4k3MHhsNPRMrD5SOAzWuGGZxtWjJtrVpgpdeY0zIx7h5v8fkE15gft2NNERPMXKtZmL2+i+ZAn+J8FbU9//LvgDTQzR3XaY4m0f/QjaLaZACRYXaoJZmWpRUwZHhvXf+Pi4dn+pr4SRlWMStARcLGjB+DN/x8XwttyEb5G3bwsiBs28lILSyVGJ+V47KcOdwuQHIzmki8+loNH7Sofbe3/pDyrQcARC0pEBONwYLHeaqY9ccOioVu6wQglQgRpLp20dHMQgtMh6gMiFlvdzTDsF7wEm4QFRpBm+5CJG1RrWj41hvLooZJM8em5A9e/tJ0TDOnRWgM4vW+4eNsKHa6QgZtAF51IE997xn1aW9RvCHxLYE+Xv5+cFCu2/KbzPd7w+XP1PHxNyR3Ig/X3o2oxo+mmSy30VbQI+RK6YR2WoH6NjY1Ys6aKCnIJdslTLmUlh9K7rlg/P3zP9k5+LLWgSvu9MGzWLx6eyscOKIkaNtrZmi/7FPA1tdoyCMoEthuVz09Gy8JHVu8+TJxrN5dxex4rbgctadDcPT2NgOQeIm4NTudsRSoWi3BTNuoE+BiX7moHO8AlYX8igWmvg3GOOx9bHHkGLlb/hUUxWF9BkZuHaprgpmSlYCuomePAZVX20MSuaKJY4i6nYwUrYstJe8N1u1P9D8JYO7F+qPbCO8++33Iwbf3eLmB6cwVpvttRMuUTggSzb4WFpACtffYMDyBazGBoelpA0BsydskBSJk210jidHr188iMbH0mioKnnmTpK2RxWrTyWgosiuQsiiL5TlwvF8WFWvDEXwE0gi9ED7XKz80RMjVmlptPXu0FNis79MaQy5cu8dS2uAB/bZEL15hYUh2iKSKGoZ6LF8CdcEtvn9TIF+vkYm9eMYSxbxrZdu6U8737b2/CO970fLUcKFQGTpedSHpe/+FLsG9+nieIkYDTbCRaqDdQ7MaqLiwbwaPCT9fzbKBEneEvnTK99D1ovAbFX4/k6f0Cu9+8HCp6HF73tIx9EQ1BigrbTiqjVUV5PXj2FTAtAXln/cJ+IGMLdXQ+4hv0zHaLQchbNKzjiyRAO4aMrkOnvOe+eu52WhP6W9Wqhda58aahcRr/XEaU8Lk3om1kw/T3DyZvU5Mjyap2k6Q4Tcpi+LI8zb0a/srly1GZtnhangwxi5042ctiMAB99cxPpYAaetunm5pn1KiCfy+Ctf/VaHH/EGlz7/z6I6blFNYf84js34PmXX4HxxUWlnzwHgHLaeMgqvPkNV1j/gPy6I7XyKIG2O0/HWciY6SspaHrUAMG9t/0qVSDUtfUuRXP+vSfH685e9b7/QMH7rIAb4+d/+D1+cvNvEUWphh00G0SnClocbjyadZqrQl8RpQFjklCQtBIM3vh3wrvM8ZmG+d8pv9cJGHbwMXc19yyHJnJDETvQfdCMavKGQZTyvZq358azuZRMGAPsaFW6CnXwdlujWfHj2H07811CdHiBdx3i2jEbaJpm0XJUFxbtaBN37h7TNm4QnW1HbN5lE9xkwgYyWYxWivjsR9+PsFNHOw7wzre/B03Xa/jlz3waL3nNlWh3mE1YZsHPf8HzzsUZZ5ze03NvG2B54ANPgmSvH/sarC5BjZflvOePFLztIPtyw/APTODdMZm9Qtfe2a/pwjj3PId23/g4PvGd7+pExHbckuAzjvLL06ZKRUP1hsaGke8rOnDFJmPzxpka0ZTTRZDRQj/JtI9HinNx5+dnBaHq9GWNPOF4VAI9OSFryvmzLO8yFfIgi82zITQqGNMFYvRc3ADcVLQAOvzXCZpuh75eR5u61Mn/TTUBx6admZ7pNjsYNsSAyyJ6uQimkJrQGQu4oiWjpVLzZbkfV5x/Fs6++BkIkizGJ/bhwx/6FBqMUfJ5vPTi5+Az//YdTdu01JDQc4APf+BqHd7EjmGnx12peSU0hWZgZ6VkUdoJtd/1+/9Ig2yha+o9r/5Auavo3zPHpTeN86aef6/Xq7pxfsjMUgOf/eEPVEsnlEmTT1x5lpMeuLitNjYduQUxazOu24MPRvNMn7V61SqlQdZTl2JgcEAIILVJp11ns1Z3dnwyXkSMWB5w3NVuRvochpix4z1d5G8Rrx18SOaFnbbp/L3O77RN7eff2IGExmSlv6fAVZRhwFZj14vx5ClwKYeCNxZebB4A/y03ALqrorQ8aEXIxsDo8BCe/8wzcfYzztPnXv+5L+G+ex9WF8xJxx+HxflF3PfYE66WwbMA2FxBwb9dNQwDgNxhB85S+yhMrogNopyOqfpEwXoO7rzphympyl00rqeTpjdt6BX8gZvCd4dw0hU1MQjtSBKal0/827cwtchTlFM0eVhRjuYt0YwXYs4Do0PYfMzhOqyI5lY+OZNRNWtsbMxKmSREzMyocEJzPjQ4iGLZXIUQOmnB/1fXm4DXfVbnvmtrS1vS1jxbnk0SOwOQwKEUuKec9gKnvbSXnsDtgdIUCJlnZ3A8xU7ixHYcGw+Z54lACCWkgRAgKVOB3lKmACEOGZx4HiRrnqWtfZ/fu761pdLnKk8e29LW3v////u+NbzrXe9C7stROh91Op7akJ1nLyRufEK/EykURSYVaURXnpFb8TTVo3zNmmCxEzAD7Ispl0zrrC7bkr0UvW7a0UK+IDgmsIbrYx481cLJoVHNigXIaW1stL/7vz5g7/3QX+geb7h+kx3vHlDf28qrr7aHHnzU3jx8xOlgVVXeJVyWsS2bV880Y85C7sTO+aPxa6E9MB0Azn+88LViZUN9iRY1G7HTwiew4D9tgj9e+cK0jYwO2ugINelxEf1cLqzCKusb7Ma77rGRsYIvvAK4aeuht34YgGTalp5xmoIh0Z1SHqqyLHRgTnN5ue19Y4+iZ1JBkDayALILXACBovrsRSzk9PrJ5k/eh0UQ2WIKfzzuQzAEAVeImSq/m8gbs0UXtVlIocYnrKWp2V7ZvVufB/jC6zWpuTTOnM3lAZUC1ERGrhD6Q3iXtYs/+yn78/f/iZ1z3lU2ylBirFxFhc1ra7G//av/0973Fx/Q765ccYMNDY1YRVW53XfHbXbeZVfa0PC4VWRJbSutOldtJ5+yxD591pkl9ywnrTx9RrHbvzczrox/w2FUeZuFr6irNQTw3E/8UZVuloz4fzH/kgKdtqGhfhvo7xHPjxMERCqQhViiaLbveJ89/Mx3bISceBoR43IbGhq1wd4BASInnn6KbxLkT5P6BOkPp5vFZNwZlGA4dt7hWnDWa6qzK3VT/bxCD9JFk7xQwmvUyiWSoSNaIHikaSq2AMeGzm7i2zvxwjti8bGHDx6SLw5M3a2fa8fOPumeGkZ5jFSuYOUVVXbRP37CPvahP7OxiTErL5bbhZessr7hwVJ9YF5Ls33yzI/a6e97l+bW3rr5DkG5bXPabOXyK+zK1dfZ1DT0NLIbh68/9ekzbemyJQmjjyFFDmyJZJkImRGTKRZTvJEKPL/8wVPFLHZfKdLMFzcwG579r7Ges1X7+o7bYH+fHkplzjFx57MnHRp2fzZjX//Bv9mLr79pY1PTIhYAWHQf6xad6MTTTlYO63VkR76Ae0XWmPaBQSwmChQUPKj4IaoEDWtyKs1uhWyQkCtRq9Vc4eVZOPgEU4Jkqd2X/LMDO0Q+QtuS/JlX2aZtoLfX5+6Me8SuOCBlDWqc1Ewel0VNp0YPlrEs+N6Vl11s/8cZp2mEKcdb6Np0mV142TXWOzis3ye1nN/eah//xF/bO05/p3372y/Yt771gjbF5ZddKM7ffQ89rnurylVZZXpOGzauKrVuz14b71FMGH6pVO3Bu+TZo9bw6399ugi6U54oxrFDSsWXPwJrwnxwUnqPd1tvbxf9jG7yknBh7K5Ib8SRs6Ld9rVvWtfggE1OeH38eNdxGx0ascVLT7BslUt0ccpFhkgsGnrU5CpFnypo2iVpFyYPd1JV7SPNggZFCkX0r0pdRc5pT4gsTnoBRpG5pmI6HKsKmrphnLbE7/Ue7ylV8XwGruvc6jDHeLGEoP2xKW1rqLV7d+2Q8jUz4tHpY2hh7A0sziWXr7KB4RFt3urKSmtvbbKPf/yjtuzUU2zTplutu3tAz2DjxnX2nef+xb79wve9M9bKpAmAZbxhw7ViA8emi8XWus2ur6TFn12QUVT/mx8/W8RsVtbVKZUKzvz/38ILiJiatKPHDtrxrmMOqGRhq4xbQ0OdR76iKGdUYXLyAtQp2LRlduODjwsRm6bXbmJK7wG/bu7bFjijNlPmkxdzHs0L8k1Yusw2hY8xoN5Kfb+6psZPU6RsjAdPzRK4GRZN8irqn/NNhO93yNZzfRDCgwcPeaahnzlHLZqrQwtIFbIUs0mnz/XX5RLmtLfZI7t2WFkmFW2o7lERTGij3KgqekW7YvkK6x+gszhj+YpKa21ttE984n/Zyacus3XrblR9o6q6zG7eeKNtu/V2e/XNvUpr2bCtrc1WXpGxdetXKo2L9Yrhi1E/iawrFrw0MQPYmcD3Nz95tshfsvnqmVGUs4oAsxUewhocPLDXBgd7rRZeO4CLUgLUJp3gr6JBSnV4qAzrpazJDp/IVtj6ux+08XEXIOrp6rburi72bhpGAAAgAElEQVQ75R2nWi5fJVpWTIuWdEcmK5WpoBITsU6NjothorKsumYq1FnDahJjSAOHiD0hhsQhWqRUL1eRZXLCTl12sv3+dy/p+zBo8dke3KWWyoT5RwnWT1XS403ZwalvW2wb1q6yGvAHZt8orYJXMCZ9v/8SBxeKduXVq6y/f0TpcS6btY62Vvvfn/yELT5hia1be4Ng7o//Px+z//7f/9SuX7fZDnV1C/cA76+rr7X/9t9Ot7/+m//pZUNflFKNI1SqWWjJzKT0TsLb9CUmjoIWXpEqIkJqNPgjiYlQdhbiNWl73nzd8hUAAVM6QbW1TIScLFXUWCzMLQ8eU6uHKdpUQWaNhzc2VbRVdz8iXzvQP2DDA4MKZIBvS0UWsPKJcUX2oH20PQnmRA8Gf54ia95P/w5lZvXDe4Qr3ZuE2omQmS3X3Ly+48fVri3oGWsSfjHQykRsEOkyNWzoz1Te5Tc+eebH7NOf+JiVic8fEqN+qpW3o10z2F9iNpWCQCvaimuusy4NcCK9q7B58+fY587+jO154y372teeUoFn545bRL9esXK9DQyOKACtq6nS2Jfzzj/b5syZ4zUTLdfMBogTrhOffhLiNbGh9TMWXgUH8B3pw/6RyH+KfNlBv3/pRWtpbVSwg4hIZUWVFgUkiTcLnhxBhEqjqp5VauFFa05pVKE4YdduvNsK9XWS7oSQSLfI0tNOSRRh5qP5o4oqXq7CdXNQfFQzQUrB4kaD9IirCN9NLd+LKR5TkB3wRZzgNKqssgmdBsq0iaemVm91nrjlkD0rFq2hps5uXLfWTjnxBCtOjNjE6JBNF9OoD6EiaeEpKKmBdEjmPsy8HnwmY2vW3mgHDxyVqa+qyFnHnFY755yz7Stf+arteeNNETm33rpBa3HJZVfbRKGo3L+utloLf926Vcm3J1WwpK9TMu+zOIhR7ZRf5z+58wzI3bNF/Bw0qap8zQwpD3CCFl8gycKk/fxnP7Y6nW5Mablm0kRtOJgutAHzoNVpGukDTQnw4NOAez3MwqRduXqrldXUWqEmp46b0aFRW3jCPB/Gm6pPXjIlGnWFKZogRGAYGxcaqNl3IVGCWeUI0cQwNq7UjxPeP9Dv7ohWbIE1nutrkzKIIE3OUPqTpETGoSinqdMANR9835/amiuvtPKi2ah634gbmLfjA5SC2RMBltDHXKWNDg1IRzdcJDgF6eimzV+wPa/vLZWYO+e027nnnmO7du6yvoERe9/732Wf+ew/2NDAiF199RoJOWBl6eVrbKy19etWWyEdDA9WnV41m41DZ66upyQL7ylfVCW18DwsdGkrq/PqWg2TwALRqPevP3zB5s1p18PioSslKjI9sqYEYPBv0LMQHyZ6la4MHHSkRRPY4cWNgl25ZqsNDY7ZZFJT/qu//JDt3vOGjQGkZKkbx8hxCi4geUNC0UT2EE3Z+XlAoZxexpqqmRLqUlKB4JRE+TR2vrc3BZ07DQtOOS9WT8BMgXbirJ115sftr//yz60yBAJxIakEy3Pxh+sNlVrcVOjigQPYTIwjYDaDi0RN5LZd99qvf/Vb/QYWcV7nHDv/gvNs88bNNjw2affct0uiDj/50U/t4UeeUNBLCkxgh4u9Yf0am549blWAES4v9QSIfTNLVj3a2tN8HFkGsHr+AnyKOSwkCQlFvoUJ+97zz9mC+XNLrUPUkTkdBG38Hg/K25jSlIbkU928uYq0s2UyOoFu7op2+bWbbHQUwWL3ids3X2vNjY32Vtcxu/OpbynIms4SKnncgUw65n1oYKjkNnhw1No5wQgmkwpiobzWjXIkMLzntJ4ZzPhgXTPbSySGgk1PeD0cw/+h95xhl1580cwpUtk+gTZJf4aYQSdM/p0W7TQYSBOoIVKaDfb3ei1cQaHzCCnFPvTQl+0nP/2Zfrc6l7M5nW32sb/9qN1//6M2VZi0u+7eqef58EOP249/8gvLVVWoXeqEE5fYqacttb/6q494FlOqqDocoRi7VF53/19q2UoFptikmV/99FktfCg1lFUjLwKJYdx+8MIL9rYl80oX7sAIxREP1hzzpuqWFpRJjZU0BjjJMVIfZ8b61CQPmKbsipWbbWh4TH6Mn9+983qr1M8mbaJQbhseecSmilkrpJ1LkYeawMjQqDN3ktwqAaLy81SM8I5ZFzwQ8yY0bpPbIOAsFZhgoKZIHez702eeaZ/827+xbMYBHW3eWXNrg7vnTYre8oQLCVPuuZUTPMrLM5rS4dCtT5f2RSmzJ77ydXv+hR/q3/nKKmtorLWLLj7brr9hs7W3t9qKa5dbTU2t7dh+u/3htf0im1SUZWzBwnl24UXnys/roCVwYAY2jgifR12wF1980d71rneVXIBboqQfHAuPaNAogVoNufekff/57+gimhpqZ/htSXXaETAvd0bO7IvvBZAwO5xULyrgGjwAVTm0vNwuu+Ym0Ydj4W/ftlYkTtiuba2tiop3fPmf7EAv4gRaAu3eqfEp61HBxrn0sF2EUSeeuQKxSCeT4qNOoEy8/8y7TxBKKLdcJmNn/93H7S//x59bVZXz54Xvp8jeEb0Z90c2EbFCtGPF5lIRKfUE4ttHhocS3Suwe8fSv/P8D+3Jrz5dGsXe3tZqly0/Rw0mdO+wyeEu7Npxjx093qvnVYuSRUOtrb3u2pIiJsGoW9YY5SJH6qQP/kucwzj1EeknU/+sOmlYNAYHEUA9/fRTdvLJJ+qGCXLYcW6yEidb0bJDnDxQmbBZYzuFf6dxozHvPRZDQVW2wi5cfr0NDbvCJH7ujm3rhANUotGiuyGarrSf/eFl+9Lz38O5+jUUnWHTfeyYn6BUD4/F8YDQF1dky5ioHLku+IKZzW9pspvWrLD2+nrvLk26PCI6pA5dPcA0GCk2gOP4bvaDCqZzLDVtmh99mANZiluWJJU+i7j6rz/9ud13/yMKRCGcNNbX2YpVl1p1dXQQZ8VfuG7NRhseG9ZmbKqrs6rqClu95pq0FgCSKY1TQhGMx1my6SVqmd8Hr9GhpUnzVz/9pky92o6GR+0H33vBFi5aIOozJru+Nu+88SLFjBk834WC3SRi1nkgihjl99ko3sHhgVROKZiozsCvmaxdsXJTCthM379n140qENH/Hu9DuZQHN5HJ2LV33O8AROo2IVXr6+3zjtxEeIgALiJcFt55Zj6bDbPN6Xpww3orKxu3wnSZGD+FIqVTb2TgofC8iBf4S2QE/AnCCWLnnD6PH/izpImfNOZgzzJwwQcl+eKE/Dob9Pe799jNm7eKOs4haG5usFWrL1fU7uaYg2V21fLrQEv0LNubm62uIW9nn/0PrgyKi0nxS3AHFUeAxaSNHHN3JLUOd5/ANU3+yPzyJ98octqBQr/1jaftnW8/Tdx1ghcWlO+HooKCiRTQOfFgZgge9fN5nXOVdsUpd7NeUSJMRmcKC3Xt2lu18Fw8alcP3rlRHHTyScAKoU78fuqfw7Uc7h22TffdZ4VMJbwTmxgfs5HjA15jV+UpzVwTugbxg66TolVDy8rmbH5tld26eb3oymEVwjopABRVimmODkBxjqJZg00nV5WYupoNk1IltzJZUchp1BSSmBpK/1OKpdebdR/rtWvW3KgaAYgc+fkN66+xyrx3DWsDT2ftokuvVhNmLpe1zvZWe/s7ltlf/MWf6RoEa6eqYty74whpzFnqsIkMzWv0qbmCLODn//rPRdifzz33rC07cYnVVNFYjyKEY+Z6gCB7oi27VruQqfSQ9drU5kSlie+7frw//JK/LRSsurrGwZVCwVasuUUiAgA1oH93blsnwqWbZg+c5NNTuTWTqbCqykSxKmZscHTSrrt5i40VfIePFt0X47OrMlmbP7fT1lxxvvD3J/7pafvO935gnS0tduut14t4ETlt+HK5nOq8TjUBGqdYFLCkJOHjv5JJTaFxIHv6fHoBFAzGwMQU1AmrD1DMad0T41N24WUrFOzyzBoaau2mDSstW5Hg4qLZm2/ut1u27rKKcsx/xpYsmGvLr7rEMpmC1iWYxbMnRUe6GJM9ZMmTJaahItyhNuxPn3+8+N3vvmCnnbo0MTxc4iNStWC3KlKW6pQL7Qgpc/6+m0janBOYQt+7QI00CpTXw58bEUyK6obZVWtvsf6BARVramvydt8dN2vufHkGnRifkEzs4PPnvDrn4zNnePQrV9xcaoxQWiWt16w1NtZZ59x2u+DCz+l7Tz3zHXvyqW/a/JZ6u+ULG8UbCHMoM5w2gqJvYbyJmyC1rcSizbqbixgioiosgtqjmQ+LsGAqAPlrneipDt00akVoopXZ2ede5oTMigprqK22LRuvs0yFxyZsqPvvfcx+8eJLum9g3faOZlu9ZoW08pIivehlIe8+E8DGjJ/AFhJHIG3agLgzG1aeXWxrb5NClSSzcg5IBMghdAzfLUDGNdD53ynGng55O5J3YuLPKQQoDYLsQJ1elkOgsDdNTE/blas3W08veDX4ed7u2L5edfuKLPECVsSDLKjOcdpwG8C/nmZlbPW1G0Wj1olSX7gLLpRnM7bkhAX2+c//g0zwd773Y3v4sSdtYWujrb95re41uGhebk3zWCPVic2VzL3nhCYNHv6OSS8FkOL50biAOINvmBIXY1ZziJtc6U1bMVNuZ597qTpmWNimurxt3XKDwciLrGjjTVtt3yFK3rRHl6mCt/a6lYp5mPghYCqGKSWmUaSVgqFnz6FN4JIsgdZryjIP3bamKJECpj4nJQf0UllwuO1cMN9n8UhznNPuu4jXxIWGuY/GhdmuwLMGtxLezZq1q1Zvse6efvW7N9fX2q6dN8qiUL/WZ03RxeradVLByniaKECoSGlx1G6+eZf14S6IVBWJ5xQYMQh44aK59pnPfkp0rkNHj9rv//CGnXbyMlu0uFN0anrl8MVsJty2UjivcWrhnPvuZVUWLJfzThgBPtqYbr4DyOHa3D07WBVBb4xOdTTZlbimy8rt3PMut1GqotmsNdbl7datN6q8LZ6AmV276iYbHByWBauryduczla78qpLne8fbVJp4UMggusrtYZhOXhuCUAS6kmwGdnFU49uKfJwpJScfGz4AoEwqTpFJEmRI3xiFEViZ4m6m7a6pLaS6A+vj4fA+7LBeGRXrtxkXT39+vu8jlbbtPFa3xjlDiCRiaoZMgkjwWzJV6NQ6WkJVmPj5tutq+t4+r0Ka2ioFyO1sanOOjpa7JOfOlNmloCLY4I1IXLOZXMCmlLeWLIirpU341pYBLF1vX6XXh8m3Is30eEzG0SLDRB6dv4MQ8QYQnTWLrz4KhtJHT51+UrbsWOTwKuQTrl6xY02xgiVsqzV19baR/7nn9uHPvxBT1Ol7emB9ezgkc/l50o92ZRcO+4mYfmy1jFo6smHNxWJ3Gvzdd6tAsslpSu6UwV6iOL693kQ0XzAQkTBgw8jOnfzk1QhJj3FC2mxMEGUVq9dt8WOdPWqy2XJwg5bv+Yq158LkaCCYwFkCyx+c2tLqWMmINC77njE9uzZ50ui4MXZMvnqnL3thIX2d5/8XzpR6MjA2OEhEUVzeh2EcuuFC/NbTQydNILUv+dMW9+MiC0kD6vx5kkpOymGJ6hA7ztTxp0hiWCqBABZwS6/Yr1TyOAVVOZs584bS5ItLOoFF6+wTJlr9rQ21tt1668pSbUQJM1G61iTCLi5ZpWpIYKAaqaRrtRdWAusreKsrzy0qYhpAjiRZKeK9y4XonRMunBJICDVvLEQ6lWnUpceXpjxvr4+q63NJ/66CRCKFEUdKdPTlq+qtKvXbLajiCRZxk5/x1LbeMNqO9blFGJF3DKvvjC4ABSZS+yeJIT81a88a7/4+a89709SnpA9GmvzMvX/++99DjubmSAM8851VlfVyE3lESdOSKMTKWPIQFK5VueJ067ollUDBUp1Sh+9UMXChPXDlJcoVknXPho6FOJp6GLGJqen7LLL19nwiAsmsJluv32jmEK8fnh4zK5ZeaO6Xri+jpZmW37VBdbYWJ+yJdq93QLp2SSOXUi6qlsoiUXF4k9Oem2hIFZQ0TLPPLHTYf3EEC09iFS/hdzoJ9bLmhL2Gxv3CY4CRvyUicqcfocLUJBFPp6CDPHjk3+hpLnu5tusq3vArDhuH/nIB+3sf/h76bROTjnOz0KJbDmbNJneV71ykwX70Q//zb713A9SC5F5kakwaTVVNbZkcYedfe5ZJb8dUzV0ipl7kNqQfAqVjLPex/vrPHMQbSyJL+kBaayIl6rDWkARE7CUBhGT+noeP0Nr1sZELpyYARZxttwuv+I6G8CHp8aQ23deL3CKNHLfgWO2+dbbdVX8bltrk61bd40GNrAxSB1j7h4Qt0u4eWVR1PJZqXb4eFwkhJviNHqAE5b55y/vKEpdKqlO8QbSR2WokJoVsq7QkM+rqUDyImmjBEZNYKWO0tR2hAsI9E3pA/1psQkSiLFq3a12+FiflZcV7NzzPmMf/NM/MXYlpd1SO1OKntX/HsP1Un9aVWXefvbvv7SvPPmML1sCLthnNZV5W7yo3c694LM2gFxYdbV67Fx0AMq2F410f0HhKqlJO3PWeXze9qTYJQ0+ZuEduHLLhDXxTCe1Zycp2IgVPNjDiqYp2slDL79yvQJTMY4yGXv04S/YxCgzP8yefe5f7BvPfV/3xeZfvGiBnXvO3wvoYWGVVeF6RVObae2KjVLadLq+mfmBauWachmXzDNP7tJ9STSf+6P5AHpUak3izSXMM6szQ3LiibvNRXDS/cykScVRjEmSXlgETqmiYtKJyQnbcMtdduhIt0zW+uuusCXz5uk9AJMUF9Q4kBTyJ3yPVqXmlhaJKtRW5+3F37xsDz/6pCYS4YmVhmbM8tWVtnjRXDv/ws9pEfF3LDqxjNIwtRNFFO4+XlIkImqSK3ljI6cJV0Yc4q1UTufyeAewKXHVWeyyjDZXTY2TUBzV45ky9mw2G9aVsq66+gY7drxHz5Hq0UP3bnFpNdi1W3bZwf2HBSXn8zn7m49+2P7sgx/QhA8xmypcFSwieFqp9T4zd1WCk9lwMUJFC53EETL//JVdRS+0ZA3/jE9nN4cEiSDNFO0TaHHyWTy1IScqNLtesqOSFnXmZwnqTREP5ghUTOlexuy6m3bZocNdetB33r7ZMgValLPSveXhYvKxHIj3ElOw87kWsgvy6FxFue3dd8juuONhMVcjd6anLJ+vtPlz2+wfP/spvScPRi3XqeUZEMjTTp9Dq02dsIMo7tCdwzw4ZStpfrteA0aRhvTOLnzAk/PBQNTlgZvDgzoJNMxvIgnZqlUbNe81AuqH7tta6nK94sr1nl4WM1ZTW2nXrb7GqvMMJUjCy5p26WNbWUzkY4LVzLrwjAKMinm6cnFYsDQFK/PNf7pLZd3x0RHh7J0dc7SoAcWyMCxqgPwK4ngoY+jI5RxXTjVn2C+8nofKe0SKp0i7psb6epHppJW5zDZsucv27ieYm7Z7d22x0VHXguVzaY863tWtMnFbe6tj0gUX7yNvlpVJzYq3bnvEo/FS9cuspjpnC+Z22OfPPat0+jhJdOnILKv44+6BgI2TpDRITSGkfIg4OOvWT6+3OuHyAgQhaJVaRsbUYRvQKe8fVObIhlIQUar9Y1k23LTd9h44oh9hrR6+f5sXfjIZu+SS1Z6wZZBmr7atW9bLGmDXBBOnnr3gAgwMuhvz4pLrB0iBi6JNqilEql1iCX376/cWCWIYBshDr6eBsqxMZkunOBEWuUBSIXwtUOv8BfPVBaN8PeXamobADhwaKvlOHrgmH/NwKirE3CG6WnfzLtu3H8Jh0e697RYbGOwRT46NEf1uLmrkSo35KsfxNWAHiLSsTDoyW7c/Unp4oZbFaxfOa7eLLz1P2EOASogQuniiq2ViNuvqanXvwdlHWw8zEOLE9Oi3d3R446OkQV0xm9erkjcrBhD1WzJrnh56U8esQFFyJCCgGbvzrkft57/6rbue4rRx4r3nLmMXXrhSXAGRMatz9oVbb/BYIJl0hiV7FuLWhdgLy8VnKT7JmA3098t60mAZBaUA0aTg8fSXdxRJCWCv8tBZIE5+Hb3n2awWW8EWQgac9sqcbhqzjWaqWogSpTp2VcmspGmVIUYUYANuZMuO++2NvfsE2Ny49nKrqnJFDCL+uXPnWm9vt/h9mHuiUTBqmgoamMhUkbPjfT3Syt207eFSJOtgDx0nRevsbLeLL/mcyq0jzMqh0saJ1agSBBRzSblaOtNKrSR/htCR3FZE9TktOm3bbAoWU0JNqUGzVPhI9GtMKbUGzC/uM0rWOqmSP4XoMWZfeuIb9qOf/ruXbqen7aEHtrklmyjapcvXlizVkiVzbMVVl800iRDHJFfiwxbR05mWRWVD8qxiQ7ju3ozsCwuuRhA+876dq4twzcnvhoaGdcNNzc06ZWwAgistSNJiV2SMhPew5/IaQq+pkS4jovp1ivypPGGuBQer6lXU6afosGn73bb3wCGhads2rrL6hjrr7e21fGVOFqOmNq9AL4KRfB5LwAiQvC8SsmeZrF2/8Z6S7lygisQQcNXPOedT/6mowoNtaW627u4ebQQWX0UgJMxSB02oWChQUq48Q1dSeprN6p7AFbAexD3yqakti4VXL37aOPLvCXbmT8Ajspenn/kXe/bbz/v7F6bt/vu2CBc43jVoN2zc7nX5TMbOOutMe/97353qFR6QBtaRiEkJeaSJM5uGFVBPcJcY/IzI+wPFyzz12Db9fn9vr8y6JjAg3znOhMcaO9bVJRlSpQCa4JzznF18cadWCRiQP0Hsl8DLBXOl9ZYqfT7IB7/j+ey22x+w/QeOyjzt2LTWxidHxbEnIg+aFO+Zr8qnaNwnV/GAWbDJKd/dW3Y85sIJjhK577aiLVzQaeedd1YJU/fqmJ8WeAEekfsQhND04b5C3YprwISWxpmkBRQ5RYOKvFAliXBhDQm/T/AoboUrIThlc7Q2Nycl7kptjH/53r/Z40885fWfqWm7686bREP/2X/81h770lNpgTN2w/oV1tpSn4gkXq8I0Cj8tQLKcDnJCmhRU2XQM4yUgUiZI2OZB3etLerBpeCovb1dN0KgI5Rpako36qXHENrznBRhQt6UBSDCZcE1hVGRI6ifpxj45SjiuBLkuH35q8/Y7lf32vve/z778J+9x6oqMtZY16AuU8zf8PCAhuqRaYj1guhPmhwtl0JaODFht+583KN1wff+8Cn0zJvbYuee849Q9EvmNkgkWB+v4nl/XnXeCzDE6ywms2DYqPj56LSJdEnVskSAkB+PPJ6MRhp7KHcXrLbOhxPFEEDh/lOTcplcx+4/7LG77nncpssgik7bPbdvsInRcXvya9+2X/92t1c1c1m7bftNNlmYSDAwFctE7kzgTqCGKhKBpSRsIhBV35z+O5HWsUkyD912XRHzLT+O8lQFPnFE9XNyeRoAJEeKxnxlpcuGxulJ/eE8DFA9ImF0aWQFCtOucjHpUqUsDnGBFC6nRq2vf8TaOxdY30CftTfVCFQhnqDsSO86Pp8ty4WrgVEzU53gqdoCM2anp+yW7V/0DpkUvbLwbLh5c1vtwgvOFo8vGLNcC58fU5s0OEnux+VRsVDcBxMmws9z35SbOT16JggQp4kVGvaX5MSoafDePAusppetedppmEHiDDJlA637w0d6bOftD9oU7RKT03b7jvVS6F69dpONT7lJrygv2vatN6R+f2/R5n0JgiNeioYJXi8cgdgs2Eiix3n9QdZ4zGf/lhY+UjcJC6RZK/yd00+jfnDleEgENvh+HiILSbDFG9bV15dwb3xgCPFhmicm0wAclXLZOFM2MubBGgFJU3OTTU2OiWpMoSYw+YgHuCmkTzipOvkEZpzOyQnbftvjdrynr+QTxQ0sy9rCBR12ySXnCgZmU3M/nFriEs19b2jQQ+F/dbjU1np9IbFWgEVZaH4Gd48NpbI0zBxqGmk2nvDxVP8Omhgug0AQcYM4iQR86v2bnNR99A0M2+atd4uUQaq665bVet+r19wiS8RXS0utrVtzpahXDh+7mw12b4A4ZCkREwQaCVfC3WKlN7Jq5NqsqdrPffUOVec4NQFfhnnG1LHzAUwI+PhApSipVs3rWfyYDs2Hs+gsGD8bGurTQ6mqIlAb14Ai3gPW7vAI05XGRSnm9zEenDhOPBRlqURD5EReTGM33GSz8SR4hFTY+Jjd++DX7fCRLl+wZOoJ+uZ2ttglF39eboVNiG4OqRnRb2AToYQp7kDykTz8GDEWuTndujR8Ks+vdNWNqJtjXsPPqwyaKnnyqXQRkTqlmrhKpQwsmJy0o929tnX7/TYOUlqctju2rpE41OobvpCGIJudddbH7U//5FTxECOg00ZKuLzirtR6Hd8PX88aB4jm2ZZDz7FBMvfvWF3kwXsfe4UEh/bu3VuqrXNC+CgX7Eecr0IkR+XmExMym1oYhuPy2oxDl/y7KhUrOHWcMjVCVFRYXUOj97mn2vHSk06yPa+9qt1Zm3dql5vgKQESwqaTADEwRvTb4wLuuvdLtnf/4cBIPPjJZmxOe6tdcP5nk0q1qzlSl48TyGIp2k4Vx4CTQ1YV7r6gaYIEPThXsI7R4qBqLL4zV71FWhi+mLVeB/DeA7cibOYgdvT199r4ZNHWb75H/Yll0wXbvmmVmiCu23CHW5NCwbZsWmkNDXnXmJ+loKl4JPl6ucLUnuYTrD2IizQzYgBxJmdRvDNPPri5qFku5eVKdfBv+HR8ReSyfIh058fGramxUZOeQwUa0p/06Kp9Hhw3J6nS2tpSJwkVM77UKl1drWIOvppNIOVo2rAy5s2WVJGkLJkGBwFiJFCH08r4Ut/97p+/+8L/az/6yb8nUoSbMtK5OR2ttnrVlUltclJsov6BvpIrkwImLqC83A4dPmxnnNp7wtEAACAASURBVHGG7d+/P20cFzyk946v0RGkWP1gEHuoOFNI/HQtEtVIL/mCZsIeHh52EAslbmfwuGz5wADACmXhCVt5/Q4bROuvttZWX3WehgJuuOU+cRd57Y5ta62y0q2Gl3T91AaHD0EJAl9POJ14QeMr68kaIBUzu1gWLl2bgRMvOHNyUmkbAR1ADr6NXYOf53TqgZaViTwQ/5bWfEKmODm8BwEOE3m8uodvn3bwowbhYpSsahXxk+ZJ7EjtVhU2PTGu08PvifWik+vTJAI0UmtSBbDujMn68b/92p57/kczJAaB4UXraGu2Sy75vD7PpUhclQq0TeBTZaUNj7hvx2+KXZvJqO88AlG+R8Ap8inFGXwmQ4/QpZ10N8hmlYpXb59iFhhZfhp9ALCSTJlnL37JGihtnLDBgSERSYDAW1oarLd/xB59/DkFfOUZAr4NUr8oSxp7bDanpSW9H03PxAV54ciD7jRRUi7HSTQ6uMz7FZTr5eLMfdtXleRRiBbZaSw8lTAwc0w/1TAV+4FjBweFZXMDkiVFA25iwos2lZVqbyIXl79XLd/noHkg4mpSfuK9i4SNxe4c6utRkIf16Dp2TA+VGKMhjSP3ua/MdEWe2xEoLPBrew7ZV772zRmdPh500ayjvcWuXH6BTtro6LATRhIW7s0gBUXz3G/QpOMABOIWFoyUTGmZ6tmetlIdYFOxpG45/MTTg8c3WVjPnRl4QDXPMx9VNUPjvrzcjh3rsjGJPUyoU+bbz/+HvfTSK/aRD73f3v3OU0QjYw1k/pNiFfcUMKxKsEm2XDSwtLDMo5UGf5KlgTIewZ024z3brlV1TunMLMIgb6CHklgoBDTHjh3TYvE/pp5Ai0XjxLCz0GZXBC1JFMAPj045FZ6XVgl1Q+mivqFBwAbvAZefzhOsA12vnqZHH56f+Gw5phKs3LONnj4Yuhl75fU99qXHv1k6WREftLe32PLLztECtLd1iIeeS+NJXRfeewTpVcM/e7nWI2fSWSwULof75+HREsU4NJ4JQR6bxxnIfqLk+niPSUaCIVPuvQUQKLkmCUgkBlBg5vw+vQVo93FwYNmyOZmRg0VkA7uCd073jJXSGqVpWQHKDDN5S82sHrkHTyAkVbFkfb390jQQykpQeN8XVhYx35yuzrlzZWZZdD6YD+MEYqoxf0TGXCw3HmYrAhHMF5EvEiOcJAKjU0492d58881SH93AgOf1gXpFqzVtUJXykc6yZUEEqkwVrLW1xWe0ChFz009f/sDQoBb7SHePPfjAP5U2bUT3bW3NdulFn1WRgnQHISbwcyhU1Arw+ceOHUkyKv4wdBKS+dRg4YTK8Z6cZMQQCSxZUdI9CjwgvnJxQ0OOeoIjqObgVCf+HXT1oHFFNsFocg5DSTE8658xMjik9+BZzu3stOPHfXgTh0ULCzO5qVkHyOH0mVZtguFjR49plDmvDT4DUARunH/LJRDccWGcxDid8m1J/owXeTQ641cJHjgZHrABsLgfA3L1TkbHwStSmRUxA7B9Bg9wOggOxfhJKhli8PYOyL3gJubPX2D79r2pDbZg/nxh+MyKdxi5rtRdg9sYGR23W7c9YNAdImJnYdpbWuyiiz5tSKgA7iDAFOihIngsVlVOkKoIGIksIi4BSGZCwaSsmUrN+M8RMpqEjjk66vKnWBB6+FlUucBJ9HtqJYIk0Qj6DhNFjSd0YP8+65jToc0caJuzoMo0WkxoZOpNJMbk2rE+nOLWlhbda1hp0kDoYiIfS7K0zMYmvVTMQivwm0hzcxltysF94el7JXdGHo854oHwIVwEJx3zQIAjCDeZsxICVlvrKRraqtTgB4c89ROdyCxXRdsvc9Rm0g8eIgUZ3pub6JzbaYcPHxblGdmSpoZ6uQAsgEaI5SpcqjQ1OdCGFZuQGxoZG7ONm+8RgdHXwQmN7a2ttuLq88TH91nvHpNgTQBWlixZbAf27XV+HTBKmoAVhSQ2PPfOtej+E2DlwxfGSj0Hk+PumvDjoHYcCLlITYigquh+nWMp/AN6mmhkMSTIRBQR2AKqpgDQZ9UyVNC5fd74qSJPYvByaDra2/UssjR8pp5G75fM2uDIoAJ0GEu8J8yg8P8K7p56dGuR3Xrw4EEFVbX5Gk89in7jbAahXgzOZUGSXjy5Ovw4bi4qeMh0RXTP08BN6LSOky56kMNO5f3EdFFXicmcHT18RClQfW2dNOr5u/rFxz0VjNSPhyrAKIk0DY2O2LYvPCwlTPl350xaW3OjXXLp5xL0C7fcIV83s2U66SCF1dV5BYq4MaJ8KWwB4mBdamt9DnwaJYaPnanJ039OwJeIIeOjOvW8P/eIi+G1ZAFh2hXYJa4cr+FeuGZ+TvosskearsWfHEYWaWCwX+VpuI3CM1IbN88QYE15PYcSVDFN04TQGV1OakIt82oi5FAJPN+86vNFOmcOHTzo82KYA0NAQ15NLp9oVujEUzBhARSoaMqykxV5oF7R86Apeu/YYa5ekZFPOnrsiCJUvtfb22Mtra1aALIJ/BI3m2d6hUZhT1hn51zrp6M2je12IMSHApHH8/6UZ9ffsMuZp5hCFSMKWvgVKy5W0aeqslqdfDKfAmO85RndOFJMABBNhEIFKxVgSgBIykBYRH4XtxTxgIK0NJYb2RPuq4Q5CIhCQNEbNORXVW+fKEHEXIkvSnD1/f5kuczJFHKnBReVAtlUgJjyMKXS4hk6stfY3KTAT2BRUvEkm2FThJoZ8ZU4AET1BDKB3ukkFoulQobSq64ulWgx2dJwTaO6XfKjwnJV1TJN1My5cTYIX5HqiVLMOPGmJlmI+JnAG7FyauzwYachQcLg88gI2CREvexyfhfaFXPaBSyl5kJYpFu/8ID0dOS7U8Nlc1O9rVp5hbRfVTYuEJn7MILpwqQCJzIJAKnxca9gaQa96vAuPe4pqVfyWHhlJpWVCb93AcV8jc/VQ+SRe4Eyxu91dnbIiioDSkicov3ETYiN5fyGGfkYZQjQvVKgyXNVYSilnd6945E7VoKNxJcXrmpLimOIWJGFsFayPFUuRhl9jZk7brlKvXOc4qVLl9qBAwf0oMLH4X+5ccyc+wrGfo4IPaJCJohUzQZAlFnNQeUC2MWcgCA6AA719/dpNxK88OVRuqNOXKBvnhrr7JxjXV3H3IRly23JkiXCErhZFonNyBefic/dvOUeG5GQkpyH3qupqd7Wrr7SpqbG1aXLPSxatFjz7tiIPgfOu02HBgls/RipxQsRzHRCuTpew73weQ445YTq4fqQceX7lRWeQxPn8Bp8O6cZ9IyDwCbms0WuTPPwuKbgJuo5UuwhSE7TtLQOafCwIOxU4FETaUqT+VMVRBXDnOrFe9U3Nsq18vmaZJ3z554HUcUdPbBzjRQxyLV5QVSywgfVCfmCkzeskRqqX1d72bWxqVFMj4qqKkGRLc0tQvZiDCe4tZdEvcGClIyM4KSlJ9rhQ4dV8QIQUt2aGfSCdGlxctIlG6Cnpzfx5MgGhtEjVhwRp3B0ZMx23v6Q9Q8RiYsCJ1OPysT2bTeL0/fWWwRxXtIFTSTadnSNBgrH1MmDfeNxj6N6+N6gUVBXb6RGkQcPDwwoiub1vA4iJCDT5Dg8QUfHQjc/3AfPhoWJqppQP4KytBmi2zbiBJ4dC8e/OZgKvtM4E0G4QuSmZCUJ5KIoo98vK7P58+cp8GSj5MBfqiqtd2DA0+aHdq1V349gypERW7xkiXYoH8omqKmu1oPioXd0tCvoIjjgZKjzVcN33Q8TQfN9plRwwVTj8OXKy1nQqry+DyCxZ88emWzmx0RDJic5YFz3847wMYMWc8rNNja3lJo3dfNl5bZ9xwN2uKvXyQoSMTQt/FXLL1B2wIZgOLBSoFT544EQvPo0rH4bGhoUYKLMJevSIdFBrJsjJUq8BKGOlRVyFzx8Veum3NVMjsFBdHcZiCDP8Y9TSd7P9fm8cYUTC/dBAdnUlDaUroHa+6zysdLrRF5l4/D5mH5QVoLzUO5g4XHPXJMscHlWaOgodDYi/3u3XVsEg8YUs2vmz5tnBw4c9FNAwMaAPem1wsVjisSw+1EK/0PEBjXin/NQTznlND0g1J727d9X0ogFHQPpqqqu0ebp6u4qQbPQmzw4rJArwG9pU6UCDuYKCyAs3YpWla8tVZ686FBhd979mO0/1OWroxJrRgu//PLzFXfwu+IMjk/IauH7sFyaDZOrUPZARTIfRJM02I+NxP+AM2wIOAccCj3MfLVP1NB0aDKAvHrfNB9+2qN1FW1SSsufvJ50j4yIwJb3xcosXLhQCKiyIyZWzJ0rF8DPgvdIhM+z4ftYBtaM9+HeOHykbaScvBfumc+m7q9CESqflWzwPuvonOPj2+/ccrWoV1wYaBbzVkgdADHYfZwI9a2rQW/Cautq7Pjxbgcp1EAxba3tbfqgBQsWKdh4Y88eFTuOHDooszw27sI7oF7sUuriUaliUZubW3SiOflAsTwAuO64noiS+Tz52dS3xg25WZ60+x940vbsO5gWHuyaIQaNdv26a7QoAEbsekAkHzgMT5CT4DFKvrbaDhw8YFUpwuZ7nDYHZWDo+hcnU6kX7WRj4x58DvQpI8iD4jHQgGKMmlK8hZnTzmcr4E0NmNQ6cA9YPT6H585z4b6BxTnFfAbIHlYp6FZ8NoeR9YELGVQyFj6wF/7OBuN5UW3kT/7NpuU91QcJzsLCk7bh8BU9TkyKY0dAwwvZUUqAKP8Jqhy1uroal+lqblVRprwypwAMTdr9Bw4odyf9Q/bTOZBOoYrgiL9zs9w0sDCvJwBbtHCRHTh8SNaAYKmXacpJDIFNwyaorW9Q1B9AEzoCTz/zPfvliy95mqfGTZMcyoqrL07TrEflQg4c2K8HXFvr0Ce+kWvp7nUixwAQKrl6UgHhZHGSCHjD9NfXU2MYkHii/Pi0y6SjOQdbloVXrp1m6bCQPF/undezCByCUPrgOfzud7+zBQsW6FnPnz9fr6V3QSc1MaJwURS9+OJ1In3W0z3r2YQDaTmBTcIGxh0yZkNw0gX+5HL23ve+1379619bZsu6C4oEZUCP+CwWFFRNAgIELUmNkg/yC3YVB6/aHbXGhkZbcuIJYsP88ze+obo2P+fimhubBLm+/oeXtePnzJ3ndeK2NkXtdXWgdAM68ShO8XB5aCwOzX0e3abOWRWHYOb4BGeEijiNVblK+9mvfmfPfOP7LiuuWINWq1q74pJzlCU49s/UKm8I5YuNRHDpKaW3j+VpkEilUzYAnT/4YQ1CTNOriYNA2PgdlULTtKmY8Z4rc4YyMDCmVmlwKnhFFB9FG5nuoSGdcmIfPjMCOw4SGEfEFqxFYChYTDYk+sNSJEupM5uGU87mYkPx5VIxno3xfKlUCrm7beMVRXWKpKiWF7vSlHetjAwNe5cpxY3UKDk6NqICBf6VEmVXT7ebqrq6ks/B17zx2uu2aNEi6zp8QAtOVK+IHV6czJM3aipTqHH/xRc7GdE/brC+vtF3bOpmxdqoKpZQLJC+3a+/Zffc94SnYEp1WPgaO//zn9am6uvrtWUnL7O+fvrwHH3ErXCyiFmGR3zYMf0vge4pVshmlbLxoFg0ngMPlX+THeCKGuvqU97tDJ3pCWrt1Md94pboWKl3TmlYCqSxKirjJiYQ78l990GBIzDDNaFUUkWxaqbeLiJnoWDHu7ttlIENCbPn+fNe2igJ/Yu/x/eV7ma8Uph59I71iuoxXYJqCVwgJPb3loR5hwaH/lPbNDm8LECuPOXUTvUhuuehMsWZhwKGT7GGUFC4dch0UCiYnrZFixcrTeRm65qa/T114jw7EFN3xDdepEDUrQnIGpo8P+W9D3X12l13f9EFHBLwAfNlw4YV1tfnwBInWxTwXKVONy6GB0KARCmY6BkiZXtHux3Yu89bk2ZF3XFqA6lkk6qZos6DUfRllXINDft9oGeT3Bvv5QIJ7vOVMZGTj4zIDQR0G3FMUNtb2to9xUaGvabG2tpaUg9jTgeJg8nPAbckHZtIGuSZpGz+5RtKI1nT9agY9MW7bxQDh2I+vp03Y4FIT6Sn1tMrvx4dMyw6YAonulDEV8OQpeFwyoZh7wD0JNVHTKxGh4F5T3jk76bc+fhcKEFOV1e3zV20yF5/7TVra2lNPpLFB+BgFq0PG3D2al4na2IqjdwqFm1wrGDbdz7glOM0mQGLtOLai8TKxczjUvbt22fz5813AEO9Zk5oyDGWVFQpD8gIpvCVjkm4v44giWcDs1gyY2lapSt8AvBM6V4HBgZF/Y7TzObGYp104ol28JCPMvMEpCjAiwBOzzxZADbHsmXL7ODhIzLdYPRsVKTZOfEgkDzXqCdESqjq33RBPzv99NPlPl555VWflVeeJlNZRplY5skHNhWZ3X5w337VdwFROPljI/gCKMyubQe9mWIGN8eFUd3iQo8cPqIFBIgJuhTpAj9jgUhH4KHNLlQM0ueeWLv4IoI790e0ZdUpz/Sghn5296XkufhbfBQ3XyEKlgrRNjA0bHfc+VjqX/dCECfkkkv/0UuUkC2ItDUPjyjegy2weqwHWDhVPRYo6GROpXZBBixE4ApE1ELIcj7eFGtB4DU+MaZshw3Ha7B6vI4xqd3Hj5fMNRaD58f7RyoWMK2eX3m5pmxj6mlYIZClfqLIvTwj9PGV3X9Q8ByQeBworFkmETKGhgeEFH70b/5ve+WVPyjOwRKQdqq6+aV7b1JExFA+ThW+Avwa0uNbb71V0nalGAIRAL8DnYoNwEVxkpwckU8ivFm9BynOosULhVcP9PVrE4AVYKIo1/Ilc79okS4KdM3fF1yd0qVTukh9hEgBJKX5N/hsGh85daSU5RU523TLXV7ISHAm17N8+ee1gQjIdJLLoHwPWVNrs9OnoECNg3Hn9XnBrxNil8yyePXFokypQ8KO1g0yb0aTKpzsSNArOLYwYVXM8ZNoErJsY4oTsKq4Ew1KTPIuXFdYPtfZcUAM9yRO/8iwm+k0hgW1UVf28InaYY3405FIpnJ6O/fChfM1WetY93H78Ic/JGyGQ0j8w3VnvnzfzZpJozr05KTKosLAJ6EF9WsRPQqusDmdXjsHBZLPVOHAmzD49wknnKBAqm+AzeCFUzYF74OvB3fHPNU3NmjHHj58SJuFgUR8fmDtRNzk69wQn8vCn3rqyVrY3/3mt7ppzLI49pr5WrCtux71lqfU5oiPX778ApueZpqFyarMaW93WlW6J6BZTljQjtU7l+bJKU1i/HdquCC1YvHJrUVSUarkEjBu9oFq6eLxfJ8TqxSO/rnBQVGnAaWcdeMkFlkVJlkeOpKmZHvAhyHTJkqoJZ/rC+uEjEA0eU3w6LznYcqytLEVCiLWiOGUMd1zjHANelbm649tK2LKtFBJBgSTD/qEmYcASSBDdMzDBDtXVwupwZDj95wW0gsRKnI523dgv33gAx+wg0otZtIJV7V2UQNep+ieIcOkbYqUY+eip+NdIJHiUUNXIwUnPJWBMeH1TU1Ka7bufMS5ZIlszLVecMFnLFdZptFkkkPNuKIXlTjvGBrzGnU265y3JIyAb4+/q+w5ewxZDERQT2G9FpJoHXEjVdVE+vBytNKzEa9A8miF5kFrS6eeXFs+e9QXvKWlKU3HTouMRKoCYub8EARSLPLSclTrWFzAL1Gp4RFMOL2d95Vu0ZQHkVFj8EOTdSIGIAzUIC5q6dIThfkeO9ZtrW2tCqzA6WUVYp5qIuydcMJJtm/vXsGMXr50rRwujJtvbW6Rn2GYMKeEoGg2jEjMgCUQSlbFn34CeWjE54HbRx09KmMsWrQIEfw1NzfZhk33KkZJDWtWna+0Ky+/yArTY3bayafZ7t27dQ3KsS2NRkuEC31+0ujFtQB98llt7e22f98+neQ4XeIMJhPPQgCB4sJefWW38nEYRF4hdE49G5WF4P34s7Ozs4QlsKHkgoRquuVUrj86at3dXcIgnBQCv69OmxP8JBRLmNHHsw7Xi/VlMxIL0a0r2HZkLE3ldqSRz+E6M4/fs0GmvhJcuhzpLm+KBIXjwR/rOip8ndmsPCA8F5RnLrK3p09+n5vid1h4/mRXcZMEJVJpSpuKG+Xhc+EgVSBp+HdV2sYci4cRo9NS7Qxebgy3EOlUwKaoSjj6VWZz5nTY6ut3ajChu+FpKUlcdvH5lqs0Wzhvod4Hl8P/pHf4dnw+zJuu7m49JK7t8KFDRrDLn+oM8qPq6Bh074YGReKwd3SKUtqUKy8T0tjS1KDnxGZQYWaqIFOvAk4isi5e7OVhfs5zBDDzlBCh5xG5ymgSZfGpYbiuDfGFN65geTvnzdV1URmlkMbJ5/V8Vv+gB4gEyzzv/v5eXZMX0fos8/hd16uLmh1K/k6q45Qd998hPBQSH1zsgUOH9YFwvoQNDw9qIXmo3CSRrgMLznFTE0SxqEieDwU7P+2005ReschRueJ3Gpsa9CAYMBiVpYghlPfWeQziIIr3qhFNf/FL37Lu3gGN5NCEiVzOVq+63MYV2HlxRtBdkl/DuolnNz5uy04+WYEsmwMkrSTHopGiruilzCXBrYoLkmvUYWDTV5QLJm2sdx4iETZgEQ9atXTIGslP63SDDPb36Rr4t/x91nsTCaSPH+9RysnP+CKdw18oOG1qVpoLMQX2sFrNAvXLlidhSA9EuTbdV1LRBK+ZN3++Zb5453qNJglcmoALKBUT3N8/oMUMhg5+ROVWsWkdcePGYZLyxckFatzz+htJF29cpr2hsUkLD6QIGkdEzOsw4SwqlTEu3OFFpx+B2Olk5fOCH3kdOW0ENjz8qPVjcVj4o909CmYwr6SUVy+/wIY0r86HJQDv8loRQFP/GVbjlFNOsV/+8pfaLIEQirac0sj4XnDxFBWnDhkwdbFsUutXZwdwdFdpkUOdCnUQUctQDUsR/rGuY7oHClq8jnEr/Ly7p8eWLVuqg6EYJCFydQlt1ABFla3x/04Jw1KiJ3Dg4EEVYYjRgqcYAR0HD26j+PWP3HZdkXIlUXx0XvDQBgcGBXzgD+YBeowSJdYpNaqpd9UMomi1W/X3yULIVShSLZeZyedrZaZggAqwSDNiRsZGZbpY6JNOOslee+01ZQQUQyicvP766+n389ooLHy4iKAzcVNBGmHzPfH179qbbx0QCdPVovK2/LKzrTA2ac0tDTrZCxYutD1vvKGS6FuJ78/G5CF55uINCxFb8D3BrhMTdvKyZfby7t0lBg3Xz7VF0AYjh40xt7ND18/p1eZJaKHLrngJl3QVi7d37z4vswJIqWbP73gAzPOL6hqDk72+79mAtHlF1/LFfdfpp9vLL79sdfUNSuUIltn9vCYsYxwULI827m03XV6UGTSmOfbLj0SPHHktfie6QgFYSLWYncb38IEnnniiHT54wJYuPUk3jAkiAkdJGk1WPmTu/Hm6gFdf+YNuCBkx0g0elDhwSVQAHxQRaNCTeFj8bgR4InqmICjydn722JPP2t69B0XChEgBVezq5edq4Wtq/DMwr4J5wctpDKUMevRoKSJHn0YpHOzXRMNS/AOBIaGSLBTXwCmlhkA0r5gEhJD4ZWjAq4h5ytfHpQg2o28LXa22VE2TC1Cw6ILIuFYWnqZLDpqKZJmM+A5Y2qVLl1lbW7v9fvfLugZa0kBbeR8KbFgv6OgLFsy3ffv26nPASThYUeDRCFa1UG25poheLaeeKD4wXo0T08NCCWtMgYMP55vWCBE1WKZmymmEjxgSkPdZsyBi4qGlliWoSywE9fz6hnpZADB3AidGjfUPDBr1gNjpgfJhbQQBq03awRlAkGh0ZDHxo2WZCvvmd79vv3zxZXHKYdYCb1512XmWLfrkCLmmRElSPSHx491v+8PgRPGemHwCOSzNbJ8vcIh2KLV5eZ4PM1fl5rExzXg7uH+fglI2GP/GXLNp2GQqG6fBSNGHCLuI9q7ow2NDAYodOHjImpuaSvGGqF+ogNBJm2TbyPe5D96bTIwdxqYjHti/392nGFKDrunPa5llK32ie29dUSSvFfm+ucWOHT0s8QB2fwj1xWkTzxwevSpzMzIbUIx54+a2ZlGCqem3i5yRZqAxpntoUGkh/vTAoYMGpRvMnx3Z1wfu7L43SrpRP2YjCeYcn3SZlcRa5XNYiGE06spy9h8vvmTf/+G/C/yAZ1dbU2Vnf+aTlq9w5kyAUUDLasdGIjU1kODmRPzUTLnUHpZ8uNQvEnE0zCaY++EjR5KlchYwGQInv6ba4wi+x/1Qv4+NvGjRQuH/PEOuHatIDYMNzgKxgaLMirVgERU/JJYubOawklw7B4vf4X6Ih/hZBIsE0Pwu38NKidUEIol0HPf44PbVAnCii4P55OTumOkaATW0D3t0yf+cAhC81994w1E3RBCmXU6EDhnBqML3qyxfjVBCmTU1NSp9ES2bnH98rCRH4qVCJk95vRlfxHuRu3reXukl09QCxabDrImGVVll+/fvE3y7+4299vgTT0u8IauFr7ZLzv+MlaXxKVTBcC/CABI/X5Tkujo7dOigTjlwJ1aOzIbXhK4di0MPH0GbyItJ5NDr626psHJsRip8AEsLFiy03/zmRS3k29/+dqV6eu8JRBXrFZSxIKR2xC08B6hgArTGx/VZvAfvSdPo2962xPa8tTfFOs5o4pl4EDolCBpLRPEMXOOll36n5xcnPdwGyqWsRWbbugvVUEEKhQlBQlMPRHnhuI1PTAlp4jXC4EGOxD33Sc+8uQr7CdQJoqAujLZdSYVOKpI8cuSwAsXDR48IyGCnc4qJKagtc8qxKjRa8jvisA8Oq+yI9RBF+m1L7K29e62hrk6Vw9bmNqVik9Nltv1OKnSwSgtWV1NtV1z0Wf6hoBKzPFtiFPOIxUEMghNI8Id5F0rZ1CQSBEN8hQam6pznw4OJPu5ZTrOwWAAABvFJREFUTGDvIHROBfCYJEqgRNtsXII6CkFtczpkesEh+JMvTj6nSzP3VCHEZ494Kq1NjwrYkAYl8jwbG73rlWfMurBxJLyUAB1laalbCYvgKGWSgU+/l9l+/cVFpLkwt21trfIvqnc3NGiXAtzQphMa7ZxoatZAlbBOojLEQ+ADeRBcAOkaqYMHRpzgCQWCwqKtKL5Z+G8CSJBCHoT8N0SDnm6dlob6Rj3gI4eRP81aY1uL3r/ryFH9WZUDSCmz8SmzGzdvV9Mg9KeafM4uu+AzVsyWWbWUpt2PB4YOTCuzy8ad1TDJ94Jq3tFBQ4e7lEhf6d1z7MERShaH9yBd4/5h33JdsSFU+yZAG5sUlgDKScyDBaFphA2BWed5UzvH2vL5xFguFU9KPKxaw/HeHnvnO9+pcSxYXiy1KqkpLS5RvmYri6eFn03OEPSNjxdAAfOSC4S7pTbfKevp7VGKBuEShA5fGcIIAV2qNJoeaHdXl0622q5BqdTsT8BHKbU+FS/qrLe/z04++WQtPr/PotTVNSifR6eGWvKRw4fTA3YtWKLd4eFxa2pDdRN/6Pg7o8zkGianbMfOB2xkytUr3vOed9mH/sf7LFfmvWlsnkgh2XD8OzIIrAlLywOONDFSOR4498TrMZEshuoMtEez4JWV+v67z3iHDg3AixdVvPERq4e76pw7T344MqTFixfJXfG7x4/3yvJkyp2AEvgIm4nMig5dxz8G9WwCKY0iFu3nsjKTE3JP3O873vEOcfkWzsciHJAb4Xq4LjZV5s7NVxX5UHwPPogTTQ15/779DhXWNyilU5ExhgmlZgF2rwgEaUQJf8eEE8k6ScE7cpyPRp8d+Wmda8tHg37C9slJA1o8/YwzlGcTmLS3z9HD7ek5btlsTvPtcQ9DQyPCEQBlvI5g1j80Zt954Yc2p6PFFi5ot5amZsunFqpAwBSApdZh3pdNRZFHRNNUYAnXFVg69+DFEidYsrD4V96Lf3Pdbz91qcz1q6++6n15GhA8LkugBpMCJW+v2EEqpTNYm3loWEr7YskyRSs9D16HYASvI4/n8/k8ov5onuBzvf89uIbetctXXC8CDX64YA6TXeS9d45OGrUhJ1YoJowHQu7HLzQ1tSQz5PNWPJhw3pZy/ELBWaTqb3Mcm9ewu/g5fx8ZGnS2SL5G3ZpUjCIHp3BAIAN4I1p1olmJk1dWJloWppj3amlpSxOovd9eqhaa+Ybahte6OXHeIQOciYS3B5R8EcCSe3tFi8qYVx65F+IINgHXHac+ImbftB4xhzvq7JxnR48csSVvW2y/+MUvbPHCBXpf5upQZqbRI049+Ln4c5U5mzOnU00msHZEBqFRNV+tE8n6+Wn2AktM447NiushnuF68f1oBcxUL735MrKgzg5Suv26bz4jJGe4Rlk6miZZdGrF+DOUKKKYQD66YP5CmXmfHu2Nj/gYL0WaokgCQ1XUph0z5mHGqWEx0cKXJhEQYxrnIXp2InZwgbyO3yO9w6wRaFEDj5vmmubNW6A5LgRAMHz5OYvOaaUbd+68ufbS715S12N9nevToLXHfYHaqfxb6uwdV0ApBm0qnvCQhN+ndIx74Wfcc4g68vv4V1q3+KKoJe5bf58CrUWLF9jvX/q9vfvd77Gf//znej9cBfcWamCSXU2jzvH1WAbFRF1erGlqbhRtvafHadFhBaiJ4PP5fK6ntbU9PfdpweE8R3EUYCtPeqDKCef9sTqk6/xcXUNP3HdzkZSGU8cNR3QI4MIJoFIlKtE0rcXO62bXExEvmDvPiQzlTg6I4gUXyqnhRr1Jo09/Bh4gaDhNV+CU4tvhe+MigpoEygYqxfu4C6AChabulDZM6NFyoufPW2S7//BqqVWrrtaFF+hY5T0nJrwVKXJZpoY5ROqyZgI2YNGWO9jBZ6jXL6lhuTy74+xBjOT3+Z8TxLOb0+6Wq7mlMal4e4eu9/oPG2JEFLJACjHv3Bdw9euvv6YYQPFKuReX2Ozx/vxJ3ULo3OiwGik62zt0kHg9hTUsAxuUplfiJgFrYfKnJ62ttc06OjqV4jmHcdoyO2+6rAhIAbAC3iu0h2pRahkGWXPFZ4CC2pIejqDMcl8U/G5UzXhg7PJgfCiKT6adm1C78+SE0LtIMXpT+dWnS7nsGj8DSJJ4YqI6QzKMmXFhJicnaSHK+/yY9OCERasbZkhB5Eu//40eEE8rfDrXiRuJiN3h6Ua5HDD7mKnnCCSl0y69ln/zu17r9tHoqrZJ+AGk02vkyIuhvBF1dgQLuIbe4z0lxhKHQSVwMZCnbJA6SNKpjYIQh6e52Z/HokULlAIDu/K5R7uO6WBSyeTZxrWRfkd8BTfQp0zOVDsJ+v4/WJZZZ4vk0WIAAAAASUVORK5CYII=">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -684,7 +723,13 @@
     <xdr:ext cx="304800" cy="304800"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="19" name="AutoShape 9" descr="data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAO4AAACzCAYAAACO/iALAAAgAElEQVR4Xrx9B7hdZbH2u8ru/fRz0kkhjRBKaNKkKCjGC4JSBEVERLkowgURFDF0RQREpLeLqBBCk4RAekhIAukV0nN62b2t/j8z31rn7ES8/733+Z9/k8Np++y91re+mXnnnXdmSXNef8Lp7e5Fe9GE4QAOgIDfDwUOZEkGJCDoC6JarcI0TehWFY7j8MeUFgVnTWmE6VhQIYOebFkmbKsKwzDQ0NDAz7MsC/Tw/u6fvpZkSJLEz4Gj0v9g2zYcW4IMFTfe+Av4/VFEY1E0NdbhlJOOQ1fBxt7eEtq7OpHJZVCsaNDLVew90IlUfT1s00IoHIJuWDhQigDBekh+P2RVhRrwIxQOIxAI8HN8PgWKokDm07XhUxVIsiQ+w8GktjiuOi6C+qZ6xEbNgG6GseCD+Vi0aBG2t2eBUBKOraOqaTB1Gy8+di9kW8M11/0cPUUdtiNhZEzG9791DqyqiY1bt+Hj9Tthpy5AJpNGqi6BUqkMNaDDNC1IjgRHTmHbrl3QjT4E5ACi4QiGN4RRV59EPBFCa3Mr0uk0FFnB4pX7kSlbKJT3IKBYsPQOSHYJFcNAUFExcdp3MdDfiaOmTESxlMX0KWPhOEVEohYCko1oMoU33liBbNGHxi9+CTvrfbhg2hh8eKCI7v4sUqYExTIxkOuB0r8XqR1zsbXhHBx53NGYEMlj1iWnwDJN7Nu/B3975wN0ZDVojg+5ni7cdPU3UMz04Y677sT4YSMgWRZUWmjLgGQDsB1ICqCoKmRZAiwH9B/9oz1A14WvigLouoP2TAH5ShmmBfzp7p/g5OOnoVAoIBwK0VblPSY59Fwd5XIZjmTRbuKtJdF7ObTDh/ai7dA+Ez/zfk6f6eeSIiMcDvP7K5IC09Yw85qHUDT8fJ0cxwb9pzgWTEnBV49twN0/vxbxYZMB00CxWISq0N7y8fnRsRm6zucFiXaWeNDep9/9V49B+wAgyzKkt2Y/6WQyOWzp7Icl+wcNl1ZOoSdIEhTYkBUZlUqFl4CMk96IDDlabsdV5x4JRRGLrCgqLFODrmmQZBmpuno+SV4MOuBDFoh/DmnQcB1bGXqeA6z8cAU2bdiK5uZGdij19Sm+MJFkE/Z2Z7Bu01Y0NA3Hph17kC5U0DOQxojhI2HoVWiaDsu2sb8UhRRuhhwIwOdX4GeDDUP1+9h4fT4VqipDVRU4tskGK7MhO1AkCRObo/j+iTGkGlIIDTsaVc2PVatWYv7772NvXxGGGoVtGqgaOizdxnOPzEK6vwO/f/Ql7OrNYlgqjrOPGIZhbY3IZ4tI5/uxZ38Z2/om8xrGolFAlmCaVciSn51OxVSwcfsm6KXdCPr8GD/2KMiOAUmy+QOOBU3TeHNqcgTxpsNgWXnA1mDpWSRiQYwd1YrO9n3Il1vQ3t2JunAMra1taEj6AElzHYSDukQMjlXFTgf4bOJR8KlBfPmweuzsyaKnZKLvQDeGNw9HKGhDzqWRmXMPIufciExJw5cOT+LSGS1oSiaxp6MTj771MYJ2FkeGu1Ep5dE6Zhq6s2U8/sRTmDxmNMjiFIlOlyxTGJktkbMkw5XF9w6d39Cm5o2tSKjqNg4M5FA2DBiGg4WzH0V9IohSqYRQMDj4N2SIWqUCTdc/13A9I6H9WPtetYZLzkPx0f7ws+E65BYkBV/+3v0oa2T4Yi+zgbNhO/jzHRfijDPOBoJxGOUKBy+Z7Ef187nRg+zCJudSY7i1BsuOxwtiroNhh0bH4P6Ovpfefv1JJ58v4uOd7TDVAL+GLCu8ib03U9w/oMhpOxYdNUzLgmNr+NrkJIZFyogn42KtHREt6bmGaUJRfUgkkgd5udoFOtRwLZN9ED/f0DTMfvVVpJKNqEslEYtFodBx0YlJDjp7s9j2WSfijS3YsrMdhiWhUKqiohniojkO9GoVXVoEmq8eaigGf9CNsn4/G7DP73MdDtiAySh85IBUivw2VFnCqKSKH59aj1R9EuERx6JcVbFyxYf44IMF2NOf5WhuGQaqugbTsDHr5h9iTHMdHnr8FazcugvHjW9GW1TCKaedgo49e0ExoD9Xxd8WWFBVen8/VCXIjpIcBjmPiiFhX2cnejvXwjIKOGnGOZBs2gAWorEwTKMCmyKF4+CzzhyUSCtkjkwyRxafIotNSf98QN+BTWhJtMA2FYQiQQQDYcDRYBsSHLsMnz+AhrNPRldrAoVCGjNGDUMoGsauzl70lGRs+7QXMnQ0+YH4wt8j9MUfoGJJuPCYkbjy9DGQLBu7u7K4YUEPDi9uw1H6CoT9QG9vHn2ZAhas2o6Ro8bCJ8lQJQmGbcCxLMgOIKl05GDjJSPwHLzY3IT8FECVkC9q6C1VUKjo7NzWLnwRsDTouuH+rRtJbRvlUpn34OdFXEZ+9J/tHGS4nhF6hhSMhNiI6MOEhEy6iAtveAqGwZtUoEmpAtkOwIcy5j9/PUYefipk1YdiNjcYSQOBkIisAO/LweD1OSGWtnZt8KX3ONRw+ZjemvO0o5eKWLvzADKmD7Lih2QZcNjKIUI9LSihGItgnA4TCvyOhiObwzh5HCAbOi9sNJ6ETl7MMGFZNgxDh2QbUANRROMJOA4ZuwJIBrmHocgqy3ywtkUeTHhdOuAP3p2PSCSCRDKBcCQElY2JsQW/1qKFq2H7gkikUti4uw+VchWG7aBUqqJa1WHLEsqVKhw1ii6jHlI4igBB5HAIql+F3+eDSh8EiSWJoy5DZFlGKKjycRBSaw368NMzkkg2tiA+9hhUKj4sW74c8+fPx/6BAuxgHJZmo6iVYRs6rr7sApxwxOFYsHgNnn11EZriCqaODHO0PebICbBMA7v3d2PJOh0FNECFClMvwbIcyKqCgBJCsVpEpH4kdu1YhkppP5pSDYjF63DFhV9Gb18/PtvdiXK5gmAohO4BBUZwNPyqCsumjUZe20E0GkCpWOHXHejajrp4HVQEoUoyTNPgcwUIIZl8/kWninG3Xo3S/t2YOmk8DEXCZ305pNM6KrqCge5u+GIJNMx9APqkmdAiPtw+82hMa9QwqmUEdnXn8KNXNiNo5zHSOoDj5U0YGMhjIJfHkpWfYvSEKQio4Iir6yZff1Wha2ox5GenLLsGYVJEk1yoTNtFQrZcRW+2DMPUeS+u+eA52CahP7DToy/IGC3bQqVc4c8SuUk3Onohmd6XIPOhhusZI6dpcBBLJIZMyzbx4uyleOqN1bAc4VzYJmxyNgZGNIbxyu8vwvBJZwOOD6V8cdBYfX6K2oBj2xzMhgzXTQ9duHxoQKu1axGFh+C09I83nnEqpTJ2dfVhX7oMS/LxG9hsHAJPB/w+vrDk4WWJFkNGWyqMeuMA0rksdn66E0FJx29uvgQWG54wStMyYelVmI6Ozv1VTJwymhfRkil3FHBI5CQyDIMWmAxXZMtbt25BYSCD+vp6hCh/USWOtF6ebNkm/v73f6Bp+CjEonFs2NODTDqPctWA6g+gVNLhyDIqlOtUHKT9bZDDcTbcSCwK2afA7yeHJENRZAHTZN4f8PtUBH0y5/h0nC0RP244I4mG5mGIjjkKhhnCwoWL8N5789CZrcAKxmEbQKlcZHh03lkn47KZZ2PvgTRu+vXT6Ow4gNOPGQ6fz0HE7+CwEcOQTmexaUcPDuTGoqrpkNUgZN7EMmQfIQoTajCJYv9OdOzbgFhYR2NzE1qTEVxw/plYt+UA1n2yw82f4tjZVYaqhGHLIYEiZAWOJMPHMM2Hgd7dGBjYiqAPCPqTcBxy7WLj0LUNBANwNBNj/u1ctE6fhnFjD0PBtNGXTqO6rwOObaA9b0DzBeG89zSGn34xtvRm8eSPv4rprT7eFzs687j6r3uR8pvQynlM8OUxrOt9+FUFz85ejCOmTEDYrwjD1UwOQbQfac1p/RlJ0abgvUZG7RPBw6fCtG30pHNIlzQOCC1N9fjHK79DtaLB5/MJjOZyL/S3lNZxoIEFmwy4ZuMLwxWG5BmLB5+9/UVPD0Wjg7CVHOH1v3oaa3emYdrE8QjHQq9jyRK+f95R+PGVZyI54ijYugWtooljd1MA+to0DE7dPCjM8Nt9/N/y3H823DnPOJWyhmyxiNU79sEORGFYFixb5Ld0IsGg8Bj0vSzRgquQLLGABOvWbViHancGC5+5FgHFgcMeX/xtuWzh+p/9Du1dFVx2yRdxxcVnwaILpci8sLyIJkVb4U1sKCBHsmnTJs6bgsEgX1QLdBHEg55pWQbefON9JJtaEAiGsPVABu37OxGNJeFICvoHcgypOrr74PMFYDWMh5JoRDAkDJciLm1wzuE5n5XYcBWZ8hUJAT9BOkIHNlKqg1vOaURTywhExhwFywxj6bKlePfdd9FdqMLwxwEDKJbz0EwT08aNxi+u+y40M4CvXPgLZPN5HD0hiZZWP+pSKUhaGU31dVj38VrsTsexZdNmtI1s4Yt64EAHHQRikRjidcPR2DgRDQkL06fGMG5MC1paGtHc3IC/vTofjhlCT08X1m/egZIdQH/GRDCsMtqhTeVXJRBMI5YiHE2hr7sLo0c1YOP6tUzYsHGoAeYi/H4fZNmGKsVx5oP3IkBOLRhAbKAHxw68i5FNCV53XcvjP19ZiONPmoGGuhhOPOdCdGUqGDlsLLLpbmzZ1YXOTAk7uotoVVU0GxvwwdJ1eG/pGkyfNgXRoI8Nlxy1iFoUBhzeD2KPkVEIo5JlkfcyWaXI6BzIoj9fheRYOOWkGXj0rh+jWCrD7w+IvUEGBQeWaaFULonXc0R6d6jhEkT3jJQ+e8fiwXQ6nkAoJN6fSCjbxDeu/QP6SiK/pSAmILcKWSrh+TuvwCmnngwn2gSjXIKpCV6Hoq2XchInQScnzon28cGG6x1DbaStNeyDI+6cFxx6wXw+j1XbPkUBIZiuN6YX9zwhQUpeG9vkjc4naBv81rlcDls3rsG5R4zAb/59JkcpQ5ax89MO3HjLg6jqfui2jnAwgCsuOR0Xff1USGoYNhm4ZUM3CbbQK5Gx+HDf3ffAMmUR9RQFyUQCDY11aGltRENDHSCVGWqt3/AJLKsevkAIn3VkUawa0C0H+zu6caBzAGogiGgsgT3daQSaDkcw1oBgLMS5G0UYiqzkrdldsPHK7HRoC8mSLTavLCNoWbhjZhPaWtsQHX0MNDOMNWvWYM7rc9CercIORkDeqGIUoVdNtDbU475brmMS77SZ98ExMrju+2fh+GmT8Lc334Bsy5wv+n0h7O1K4d0P/go4Oh8T5dm6XmGSLxCIYerkmYDUjWggjRt/+h0E/UFOXwgmd3QeYPZ007Z+PDdnCzLp/TD1XjiWAZvRggk4ClQ5iFPP/A5WLF+EaUcchfXrP4Bl98Mh1FZDhKi06UMxfP+Rp2GnGnlNRvRvw5HlZYgEAwhHVISCIa4weGzvmKMvRFHycVWh78AO9H22ktezq6sH7fv70JctYf2eHDZs3I6Jk8chFgyCAAXBWK5a8FoLR885JuVvFCdti9MYj4El8NrZn0WuojH0v/m67+HbF5yOYqnAzp1gr8cq67qGarUi0JxrIl5kpc3PP6/Jb2ujrWcojDTDIjclY9MNA1/9wf2oaH7QVmXiSZahUOrns7Ds2e+jZdJpUKQQCoUBSA45UMtlpcXL0LWqfdQa7ucZa63RikA4hBCkd9940aGDIGZu+9792J2uIhiNI18sD7JYnD9wDkjQcsg7yQx3KQoDH320HAFNx7Lnr4NlG1i6aCneeH0V8mUdVd1kOFhiRs3Ed751Fi666GsMMYjrEnmKgObLl67EiiUfApbId8jzOZaNUIDIJAXRqA/1jQVEo5R/qEjnYgj6QujOGXh35Qbsbe9DIhLD2LFjEI4nsGnbLhzIO1CSwxCIxBCOBBGJEUnlRzDgd8+JclmBMCjvo+iryjaTPcQkRmQHd3ytwTXcY1Gq+PDJ2rWYM+d1dOU0WMEoHEtCSS/BMYCgLOHxe29lVHD2hQ8iFAihpa6Ec04ehzETJuAvr7yJdRu2wLJUnHHmJZj9+n/CsEqCA6B8T6GNHMDxx50GvZKCjh7kM/tw0w8vwbhxTcTxIxJOoFQsorOrHZt3FfHsnA5kB3bBrB6AY2XhEPPMgddBou4whCPHIp85gKOmTcWqVe/BsnshgQi8Wq9v4oSTvoThF14Ju60VMSqNZbM4r/wGI61EIopwKMjGRAZsWjZGH3UBuopVRPwhdO3ezIbbN9CPnp4+VMsWduzpRE5twOqVqzBlymTEwkE4xH0QQeVufoLSTKR5ZRoi3QjJ1+xmw7LRly8hUypRpQXP/PFOHDd1NEdWMlwRcYVD0DQqRwpy8vMMl1/ZEsTUoaUgj7kleO4nppqDlYWiqeC8q38LnegZm/JziqiCT2gIGnjz6evQNvF0SE4A+VwfVMnPTt/jZWzLYkL3f2O4IuqLGO2t0aDhUk6QzuexcnsHlGCEa4CcIzA8pg1NueAQeUAHRAYlfCYwMNCPLRu34sGffAUL5y3Fkg9XYFxTBD/4xnFQ/SYK2SoyuRIMUwGR180jx+O4U06FYzkwyP4p4beAmd+6FhWNDlCCTBfCshGNRhAKKQiHA8hmswxnJRAEUeD4FZx53CQcNnY8Hn7+TRxx9LEYPXo0ksk6xJIprPxkC95atBZWKI5gJIxwJIJQJIJwNDxouGSoDJU54eJ/8PuEU5HIcCUHv7mgCU2NTYiPPQ7lagCrV63C2++8jfZ0BXYoCttwUHEMmBUTsmXixT/ciXKphPMufwTZHHEGQJiIp7AFxwxCkoKgYF8fj2Lfnq0wtDwzxQ50Jl+IufzmhZdh4/pOpMv7EAr5UBeuw+XfPBqpxggTTMSyU2R55fXVeH89UEjvAcwydG0vR3AyWhkKxk8+DwN5BY6RxfRJh2P5h+8CKMD2nIVrNFSrnDrpTGRDEQw/YwaUxpGYFtfxZX0hfD4LwUAIkbB/kBfQdQvjZnwLOUuGrRnYtGoxunYsh2YYyGULyGbK2LanH+VwK3Zu24wxY0YgFgxAdmwYZAFknLbNXEPtw2aoLwgpLxoaFtBfKCNdKDCBOeeV32FMYx0q1QqCQQ8qi/JMuUxEnyhZ/k8MVxgpQXSZ0yjVI5UcG3MXr8Ksp5eCDNCrnBA/Qsjm3uvPw8wvTUW8ZSpMXYamFSDZxKGI8io9n2yJUqH/qeF6rPY/Ge4/3vxPhyhqgsvFQgGfbN6BPtvHxIa3aH7Fz19zHkJ5oELlIsG6eqUf2ZGxZuVHMHUDl55zLK6//EuM9Z1KN6qVKtKZNDID/TCrZfhVGUEiqIJRjD3meE726QA7duzGe6+/jkJRh6P4YYrsBrFoDMlEGLG6FJcT6PndPR0wDBnwJ5Cqi0GzVVSUKKKJBLPb4Vic2dLO3jR+9/SbgD8GNUL5bQzhWAThcMhllVXOuchz0jlRfsvVJoYmJp9zQJVw/8wWNDQ0InbYsdCrYaxavQJz352HfdkcDH8CtmGjajswqzpM28LLv/8115Kv+dmz2LSryMgkEkkg6Bfwj6KN6iM0YbIoISL72UkRdFdhcU5HHrp3YACSkub6X110AlQqwTJBSLyAhWRdmNnskjQM7fu3wC8XUCz0wrAKgK2zcGD4hLNRzNporIsjEVexaeMKhEMqKtVuEKwUD4KpKUyfei62bfsQM0b146YbLkYIKnxKnllbZuOJA3DJvELFwLgTr0C2VOVIt/wfrzGZVs7mkS1W0NWZRY8RQFaz0NXVh/EjmxFWVdiwYGhVvrYE+wXxKQzGE+uw3brf0/OqDtCbLqJUIi2BhGX/eAqRoALbMvm6kQPgNbFtlIqFQeKJN6kLj5l7oW9Z3OOWgtiwDgaq9BpUzQAhH0eBQSjxlqexp6sA2ySRzJABUgBe/vSPMGriZCjRNujEJrvkFeXe9CAcRdeb7clNTQQpO0QO1gCfwYMZKgV5PyI7ETm39ObsFxyCFSRWoGL+nvZubOvsgy2LNyXoKFFdlxhPiS4veUg/wxOCuLTZaAMR2bBl4yZolSoOqwvhtSdvhc8JsKF7LBoLZajUxAdNsMHi8o1eLsImn0BMo15BVTNQqlSYVKGLwlAl24mBgQHEQn7s7yshFG+CpgbQnzagBMjRCOaRVCrJVB0Un8rOiC7nDb9+FAgm4YvEEXYNl45fCC9UdiSKsF4mSjzhCUt7HKrrAg98vQ0tra2IjTkWphHC0qULMX/+BziQLUL3JWCbNsqmBVMTkeT5+38JvZLFc68sxe+feBeRSJyFDcKLEyynPFeFY5oIKn6komHOa5nIcCReg3JFY9hnoxO6pqOx8XD4fZQH+/nYy2XaNhZylSL8yeEY2SzhxceuRkXTUSxXUK7o+GxnN+56aCkG0n2ApaM+kYJjlZmIAqqQ5Cp8ATp1A4rUBFluxuYt7+DbX6jD5ecfjkgsCVkRiEt4NPcYAZR1C2OPvwIV00KxVMLcv7+AysBeFHI5FEoauruzqATq0ZMrsUOvT0QQpCgrO7BIrOJCR495ZUEEGZXjCHRHXArVYh0gW60inaf10LnKsXzuU7BM4gmEIkkwWsII8/ksfy/qwHSeLpHkGS7tWfd9DjZZfia/XiQcgUOGa0msirrkhkexr6cAIgYIGXqQmljy95+5EiMmnQpHjaCSyUNxlYB0DuyU4HD9VhyPeLBRDuLVQYL/0MNhJOgFULZHlx2X5rz6rENJM21yqn3mixUsWbcZlhzgheMnkkzQ3VSkcmEP5zgI+Ag2CW9JBrLr08/Q19OLsKNh5euPspqEuTPXy8jMwokDIWN0qKxNTsiWUJUcKJTbUCQmL6dbkH0+UViXJQSkAG6+6UZU8n24+LqfoOyQ2siBZDgwbR2VquYSHvQ3VI8G18wIkl13+28hh+rhT9QzxR8Mhxl+E5PKG4QgJW1OVomJTcPHLAlYpCoSfvf1VrS0CXLKskJYsngB3ps/HwcyZZihOi4BlHQTJknaHAe/vvZyjGprwPtLV2Pb7j5YpgPTcGCYFtIDWVTKOspGGZV8EX1d/ahLtXA9WcBHKtTTcx3ouoJYjMwzj0J+AKbhhyrH4Q/4och+2I4BWY1AbRiLpoiMvz75HT7eQECFLSnY9lka37thDnp79wOWiZCa4DTAz+UuujwCTdF7F/ImLFTRn/kYt1w0Aqee0IAEIRN/lEk7TmBk4jkEE7+/ewDTz7oWhaoBzaji5T/9AXapm6FqNl9BoWgiMmoSPtm8BZFgCFFFRpA2L103xxICCTcKUTpWy6p6m5UdmSQhU65iIEdSR4ed96I3/4iqriMYoDx0yHDpNSnieqUhQlK8prT3aiIuMc+f9/AMNxqNCqEk1YR1BZfd+Ai6shoss8yyXK+Oe1hLEK88eDlaJ30Ztiyjmi1wGsOkrquWMmxxrrXB/X9iuJ6he8fL8Pmtvz7mFHUHFc1EqVLm+tf6rbvQm69A9gVJzsIqHM5xVSFpZBgj0cUX5RQhxwJKxRK2bNkCx6jg2m+cjqu/PZNPwjPcIY9BjsuVmx2iYZZJ10nqIVa2uAbEb+hg9it/weN/fh533XcHjNgw2FSy4ryBlFyibkwPikZ0POSMtGoVT7/4KjbsLiLUkEQ0HkcoHkUoFB6MuMIjk6xTASlj6WvWzhJ5IQE+MtyZrWhqbER8wrHQ9QhWLF+MeXPfxd68ATuQYqOoUv1OE6TI+eecgW+ccQIKpSzLIelBx0JsOCl9mEF164tk6PRG9Ds6hXSuhFKxikymhP4BjevDp37xSPiUMhzbh3S6jIFsDh3tnejv70P7gQFkzDZEI3EMawghlYrA55PR2tKCiqni/cW96O7fCccwkAin4AuG4VcDzHIqfhlUDqRlLJd02DCRL27AQz8cj+mHUXpBjs67znSph67JrgM5TD/vGlimjWK+hNee+T0qxQFUqhbGTjsOXekqetJpLFm0GI119fCTcyZqjYVvQ/VMj3xhYyAipiYaUpAgdplUcgPFCkzHxsjmFN565bfQqkRaimqHZ+gkIS2XCoKpGvy5iHOsU2YbJ2XfwfmmZxQE+Wn/hUOkUVZgwkBH1wB+ePdsRnwCFVD1wWTE9Kurzsa3LzkewcYj4FRMvsYsgXRhMr2up0/mczvIWwwRg14Er/31obXbg3732aLHnb29Rezut3njFasV7GvvwNbdnZB8IRH1fKqraiHjpbrVkKqKYJuAKiKSbt68GVqpiIRcxtI5f+Z8YjDiuh5ILKJQYnkP78AlRXj0SqWKUHCoAE7L/OnmDdj+2R441QxajjyDYTY7VFcaR8ZApI4HgzivIK1y1wDuefSvCDc0ItXUiGA0zLU/IXEUOS0bK0dfCSrLBQnKCKilysAD5zWjrbUZ0XFHo1oNY/VHy/DevHnYla5CitTD0nQm2ei4CU20pSK49Yff4U0fDoawa+dOTJgwwd1gYv2IlffIBzoILoPQktimEMEwkqE6pMzFe8OgRg+dy0UiehuiZpnpQX9/Gc+9uQ29OQOmYXGEN9xIWjUIHSXQ17MTjlNAkIxXjUCrUp5HJQoiIKmgI0NS/SiV9uDF20/D+NFJ2E4RPjkoUiZeZ8GU0rGtWLMbX/nBr/jY8tk83n71JYwdfxiUUAP2dvShK92DXN8AlixchGQiCR81oxCooLV2RRdebuvVT739MFjjddFPX7aM/nyJhUGXnv8V3HzdRdCqGsKhgGhIcAk24lM0rcycRa3hivRMyA5rm14OsiMBqhmxEdcgCmoGlq3Zitsee4+5Gk4XmVC2+PfL/3Ijho2bBCXQBD2X5+OgaxIIR8RLu6UkjiT/pE8eMtxDj8OzGc5na0p23jlJBz563jF1DX35Cj7emUah6iCdyWL+ivUccYPRCBM0JLimjU1Cf853yB+RMscnch6XHUdXVxf6OjqhOCbef+5OJBNDxudBB2G4Q5GYWEQG0czqEsRwFVI1EZeEGUYpi83bd2Dz8vcx6ezLYHXUJFMAACAASURBVPBJUQRwSTJaJK/7ggorlMsYJgbyBfzi3mcRbx2OaF2Kz4maC7zcypPZ0XmyGGDw/BQu0RCsu/9rTRg9ciRCY46EpoU54r4/fz72EHwKJOAYJkxHZpaXan7JgIQ/zroVlmPAJ5G4YUhg4F0kigCs2GLn4fHzDovumRxwyJS5rUUoXQm9sEMhdyK6ZugfEWoWlW4klXQg/HeGabNm2zaqLM4nKSqRYNVSFoZEsLiC9EAOezu6kM0UOOqWKsQtqKhWC/jWKXG8P+99zDh6HGZMG80IhYT8JjU60DEDWPnxAZx79W0swunuzaC/vweFqo5cOodcMY2O9g6EQ1H85aWX0NjQCNU2IdN6knF45Tc6drd6QYdeK4Qg02NVFEHlos51XEcGXnriARw5vomjG9dwXcUUfSaexrJ0l032IrFbu/1vGq7fJ8qEkC2YtoSb73oKyzb3uVSpyzzDZqJxyTM/RPO00yHbPpQyGVfCiaGI6xmue9H/VcT9rwyXt8AhjQdS18fPObRYtOGrpo+VL5v3prFu2y7s39cH+AMIx2MsESTjJT0sRWF6iIglDI2pcdvi1/ls+6dQZRU/vexMXPJ1OinKlwnGDhmrp0cm+BFPJoSHYwvyNjA1wAgWTexFyqJlzJ07B5n2Tkw45Rw4VhimQmSGDcu9eBRlCS6JPFo0O1DB/me/fBRGOIamEcMQikcQcoUMg4ZDqQBLHsWmFBFRgiXb3NJ298xWjB09AuEx01GtBLB6xVLMmzcXOzMGrHAKEhFTJCYheK5pXPp56r5bQfXH715/G0cs4glCQT87wNbWZoxoSDDhNXrkKIwZ2YqoP8A1cDIM3ZLhc0j2Jwg6Ph9Sj7kX0HbIcAf7MYauO62fJNaktsBPZQvO+zjrcL04i23JH4jfkbabriWhDSLk6BpRC55qmUyO5fJZVKv9qGplDPQPoFx2cNzZX2NisrtvAPs7u1Es6yiVirh71p24+qrvQfUF8ecn/oTmVAphejOviUWRmARkVEHOyJXUkiKJzlE0CIhcmn6fq5jozeYhOwoWvfkEEhH6W2ouoDyf64lMDlCLH8Nk9yJSXsuojzMqcf619dta4sczEHLqvC9ISGRZOOfKXyNTFRGU9xqhMBs48eiRePRX30DzmJPZWZZzOf47Nno3paS9eBCa+Dz6mI/YhfPu9R00VBdJ/JPh9qx9zuFNQR+mwdEiW5Tw8ltLMHflTij+CKYeMRWf7t7JjCiRIvFEwu388fpYRZMAlQmohW/7th1wDBtNEQPzXvoDQyPR4TDkOTyIS9G2kM8jmUzyoVMOzZSW46CQLyIeF0JvWi5SAX3w/tuIROphGjpCreNgugw7HT/lJ/T+XnGcFo3E9ER0zfr9k+gqSmgaORzxVJKZcc9ZeGQURVeVWC3PcCUZlmTB7zi4a2YLRo9oRZSaDMoBrFy2CMuWLsG2vhLscB1V/hmmizyWmiscPP+72/nrS39yp7thCaEIpRZvGHdN6Ou2hA8NkoWpk4dh1cZdWLlhL8PJUDiCYCiISCSKRDSIQCCIRDyBpsYYhg1r4xbG1sYGpJJ13FssSSoz5HTuEtUy3dqhR76xQTuUR4quE2om4fXmHlEPFdB5O1AcarhQBGHIcJqgtIyqVmFij6A2VBO2IWNfVxe6+tP4aNUneO312bANDTffdBP6+3vx1OOPY1hTI/ykTnG9DfEGQn0lHlTjpPIdOW4my0g1xShMkIx9uQryFdGK+MmilyGZFShqDVJhMYWNfD7nGq0LlV3iiq6HMLyDO4J4b7lr5BkHrTedK4lhDEvGGd+dhXKV0Jd4DVuiNhsVd/zwbFx20ZkIN4yFSalShbgCWxBmruGSymwI9oqU8vOgb609H8QJHWLQ3jlI3Wufc1jVQUl9tYJqoYRyWYM/FMK2/Xk89dpyDBQM9pWkJgmwiCHMOk7aeNSWJgQMChe96U07O3tQGMjCp1pY8Oz9iEXpovs5EngH5RkuEyQ2XRyDI5JFulmfn3Nq5ni9xaJo4/jQ3bkX/fkydm9ajZYjzxyMtMK43UK3y1YK2EzG6+D1eQuxYOVOJFuaUNfUyAV20pF6UkfBIjtsuF7E5RYz2YbPtnDXzFa0NjcgNeE4VCp+LF0wHx9/vAbb+8qoqFGGoQTNqfZaJYG76eCZ+3/O8r6LfnzbIISSub9TkGEE8/lC2DaSYRWtsoEjp47Avo5+zFmynZ0T9YN6qICCKUUkyqGI9PM0s9Tw7UUpLyrQavgUkatFImE0NqQYriYScSSjIaTqUtxumYzFEIvFOHWIxeO8JtTU4VeE9JMdEkdwj+Bh+o6dA8H1bDqNluYWbPp0N554+jms3bAJDl1Ho4o7br8N27ZswquvvIyWBNXgqZ9Y1GoDPoEk+HjdmjStH7XwCQZYlCJFLyzQNZBHUTOYEP1o/vOQjLLYI16KQa2mBkX7koAKnsqo1nBrIm4tS1RruLSOdP7CoE109ORx/o1PcJ3eg/EWCBWpWP7cjzFuygxYviiMcoEbTTyZI+nl6UFk72AmSzmuLerTtQ/vfL2f/bcMd/+KPxEi4YdR1bFly3a8N28Bxo87DKPHjMawMRPw47teQqYE7vUkqSCdGBluMBxhY5aIbeacC5xzkLpp3/79fMA/Ou9YXHX5RXxBFDrhWqxu2kxsMJqxLCa+iBn2hyJQqNRUU+fyOEASDGzctAlrly3BUedezJMRmMgRtQpeOIKqBJmZpLIZ2GAgncGvH/pPxBobkWhqYQEGl7gIiioSZJUWlcK38PIcDchIZBM+W8JdRE61tSA1fgZKZRnL3p+LVavXYvuABiuU4IkOTAgZhhg4YFl4bNYtUEwDt9z3Z/RkM5AUHxziCwjNUsC1BFtvwIRP0jCtPogjp4xGb7aC5978EJIpwxcQm5PzYArBlN9S1CASjjeX2OS80VwJn5fzeaQdfab+Vc6YiQ+QHS7JGIZGrS01yjgfrx0Zu991xuxguEtM9GgHaQiBP4D6ZB3O+9oX8bVzzuXOrY/WbMQtd97HnUiU85KTvv7a72HHp9vw1uzZaEs1MO/Bx2I7/Pqe06RrRpvZg5W1ZKYjK9AtG129GU47Rgxvxtt/+Q0qJSAW9rP80/V+zN6S4bLc09Wcc7p1SOViMBi4TfC1RkTOgpvyGShLeOHV9/Gn11cy289+jI6VCSwdq1/5ORomnspcTyWbHyTwWPOgqLy3KXhw6Yd18Ac3FXhOdojfGGLHBc8zdGR8LWt+IA1seM5hNlbXUcxX8MxTL6OxoRnDRo/EmLZhqGuIY9GmDtz3xDuQFIJGAi4TbCZZoUyazlCAWUm6EMzYOQ727t3LTm101MHsJ+8REccRF0hAWfrWRrlY4uhBzoCen8lkEIklEIxEWEzheUPKYfkhAYvnz0NfxwFMOfVcFCkMeVDfERCRPjzDJa9Ji05tgNf/8hFE6pvQMKwN4UgMikr5uegM8vJIoVl2F4zgNxmu5eCu81oxavQIxMYdDa2iYvG8d/HhilXY3l+BE61zZXyUU5vCcG0Hs356FUa3NOOPL8/BstWrYMsqVEtlgo9guUGmJ6vQTAthWcdRDXFMmDiCHeRDz/+Dtdgh0vZSzsk1bTFKiNIL2XZQJa0vORzSWrmdVmy07ugfzyD4Z27nDDszlrDSMAoS0IhrQamDQQKYwcYSV3BB6YtM4htBlDGh5xKTV1xyAa64+Js8fGDhh6sx68E/uq14JGJx8Iv/uBaLFy7C/LlzUReOIEC6c76MDqgRj5w+oQeueXKaReIGKsWJJhbarDROSTMsdPWmWc134vHT8dSD16NUMhBx94zYFg5LTNlQXMP1Jmx4hisMxW2i9wQbNVZL78f1cR5mQCN1HPz0zpexbEs7p5GDdWbLxtknjsHDv/wWkqNPZMKwSow3iXWIq3GlkGS4hMC8CHuIQGvwnQ8yyEMY5IOjMPE2LvLJbX2BySnabO+8+Q5UuQ51qTo0NNbDFwpg82cHcP8zc1G1FDhU5yRvTOof9kwRhBMxzsHIyOgARA0W6O7u5oVsifrw9K+u5KjI9UNipSUgGo3xpIlqucJCDhLMMyFB+YbqQyQaRyQWH4zQg4YLB8uWLMa6lcsx4+RTobSOdw2XAyRffJ6+4ZJUJPRnHbRZxX/85gk4RFANH44wvb9LFFHvKpdEXEb7nwzXBu76agtGjhmBxPhjoFf9WPju21i9ai229pdhBOJQJUIPYjIIQWXdsPGTb38dMyaPRyZbQUNTM9K9adh5TdSMKSKo1DoWgOyXIUdCiPooT7aglUrY2UNCBgtVU6AHypUo18vl85xH9/TleLJEe0+/iMLcpO2q0hiSDbW4MZrynCVbjnAAzE37RF02m80w++1FQYLBXjeKKgvikDckOW8yLknCz677ASaMaMPEw8finQUf4uGnX4SP5bEW/LKD6665DCsWLMHyZUsQ9QX4fD1HEXAFCpSymIYQt3qkIh2PcPBMx6GiG+jtz3EU+/bFM3HzNTNR1g0WdXgEHO2bcqkoXqPGcAUUo2d5wp/Pr9+y8R9quKaG83/0IPZnqCwn1pgexN4/8ZuLcNYpM6A2jGGZq1UlfbkhpJL0jrKCSrksGHhP5lgb2mu+/l8Zbn778w7pL++5/wW8/e4KDBsxAsNHDceo4cNxoLMf+3uK2NbeCVtW+KIodAFcrSoVmSPxGM9v8gfDorOGk3qHHUFPdzeSQQkfPHsPbMliVRItABmKbFqsaiKpXDAYQi6bY8KDapBkzOTZQ3XxQXKKYBLlN8Qi9nbux89vuRNnnDAV4864EIZFr0ksJHlKmwk2ryzkko28TE+/8Ddsas+jeVgbQvEEvx9BP4uQgNuT662ngDZMSPLgr/vPH4GRo4YhMeEYWEYY8956Ax+vXoGt3QbMcCM3mlN5SjZp7EwVti5h5qnH4vvnX4AVb6yAUwoCVZlzZtpcZCB0Tixo55IHnR8RQRThCOoR/Ddg+2zOP4WWmPo7FQSDVJ5z4A8HEIyFEUiFsD+Txe33PIS8prNEj6SlXFvnHI+rbKJBnZwas/Ui33JkEdm8/lJO9bnrRaAdzxnTurBTptKd4/Da3XHzDTj6iIkMHd+evwRP/OVVhtMUxJsSUXz11OlY+/HH2LB2PYJcTpShGzpHVR/X60UE95AaiVeYnPTQFaVQZABVA725PA8l/OOsn+L0Lxwp8uRAYIgDsSwUC0U3PxZSVeq59R4eKTXYDcQ0sxuBuaVU5J5iOJxIOyi9+MJl93KrKOfhruHSMS5+7mqMnzIDUrAeWqHE50TP4sDE7fsSpx2i1Hew0MJzEt7hfR6z/S9sfPDHUvXT55y5763Ev9/2AoupKUeh1q2pkw9HS0s90vkC1mzeD43ADeWDPClClDaUQICVSKQLDoQifNG8aXZ0pvv374Nk6Vjy1z8ipGgiMfdOQhKb1svHPAhAhMoQC1fjHW1R5qHSzorly3Hdzb/FT751Oo6d+R2Y/DomLEkIKMhw6XUJ/hNbyR0dkoRVn2zCy2+vQF1bC5INjbzIPJrHJ5RankzNg3MEKemYKZreM3MYWtqa0DjpOJhGBAvmvoOVHy7Fp/02KoEUyztpjpJtUS23jEkjm3HzpZdh3RvbAY2YclETpjYh0oYzqefIfHykt5Vk6h7REQ7T0DOFCTUOiyYpcUSDB8kYaepAMhV1yxIWSw2jagRGtIopZxyFWY8/g4+27WSBfG03CoEKWj/elK7x0eant6G1EnBSEEJ8XWzRTMAbj8tFYs8QLPSuz32/+jnK2T5MnTIZr89diL+/+wEjCVru8SNacfnXT8Pzz7yET7dtd6cdSowcOGq5wgpKkYiNp23BbLw0NErHF6TyGJAt0IA9mthoYuHrT6AhKdrtvPRGnJOFQp5KQaJ0WGu43kA4z0AEXBaKO36+a7i0CNFIlH9GFQq6Zid88ze8LqTY8gw97lex5C8/Qtv40+D4fKikxXyp2mkX5JQ5fXHX1tM+1BqpZ7i15NihxNW/MmBp2Su3OFde9yDyGimEZCYe2lobcMrRk3iwmq364QvH8dr7a9BbKHGbmOclZV+Ap0n4AoIkYMKHciDyzI6Dgf5+lkGed8LhuO36K+AjscQgoyY2iPA+okDueSLvYD3HK57nMXE22tv34BvfvAbTx7Xhmlt+BZ17dkm44P6lI+qAJOwW8Fv0QqYzRcx69BWE6+rRNLyNaXuewkc1atfzC9gp4JXQVVPwMznitrQ2oXHKcTC1MFYuXYxFC+ZhR7+Dii/J4nMGfJaEEfUR3Pbti/HRq7tgFkUOGQj6xEhP+nAlo0Q8eudNAwQo76Q6L11sPmYaWkDjarlPlyZOAtEYjZMFR1yCspSn+ijXI8Y1KWPy2VPx7VvvwYBG8sCh+UbE6guyina5KMsI4cOQ4MTLY4XAwpW2shELldbQtRLr/PA9v0ZDjByNjRf+/hYWrFrLLXqaZmHG1HE4dnwTZv99Dtr3HWBDpbDvGS5BbZYzqpRiiYkSwjG7cJRQCKES20auUEKupENyNHyy6BVItu6W1Ya2NeWTNCBOMLT/O8Ol4yFy1TPcVWs34fr732HeghpYvP35hSOH47l7L0F8xKlcS9bpfWlAn6dFIHmrSeo1IumGorln+IP72/3if2W4k+plJ1bXgC9+4Rg4RgnTp00k14yq6SBXtWlOAwb6s+guaDyKdOeefWxwXLLx+ZmcolojDdCicgIzj/4Q1wdtW0NfewciUgVvPv8gE0FM8HMvgVvXPUQV4m0e3l9eXZFgGsE+0gvQTCgHWLhkCSKxJvitPIxYC0945KYFd6Eo36CckDuEXM9Hxv+TXzwEX2Mbho8YjmA4yOdBPoGIEq/vWLDUohyiSQ58hom7LzoMI5rqUTftJOiVANZ+9BEWzn8T2/pMlH0pvgQ0toZkfU/+8iZ8/NxWaBoxzIQ0bC6zcOSndjIvV/IJFpfbJCUbdXV17pwkMQ1C6GIN1j+LlkMH8XgMlk11VAWBEMEym6NDPBbj802NjmDBgd14fv57sG0xVpSWmssr7tpQV5qAx+I9BvNaYtTd60ENDExCsx5UuDF+rivYp/N9+sFZcHSaNAG8+tpbkEJ+TrF6OjswvDGJpvoEfn//b5FnKEkbW+FZw/Q63JVFY13IoN3ha8KovZxQ1JlpDwxkcihrxIWo+Gj+02wQYkqlkImSsWpahT9c6onhA0NlrwTEsF8Qp0OBwav1iqBAxBR1X9GDHP3jL76J1xbsQKFcAKwAbNlkNv61h67FscdMgD85Fk5Fh6bTNXZ4TJD30Fwya8i1eNLcg37C3zDicaW7tbCaf1ejiqwNbtKcP1ztkGiaCu0GVNauHujoga7ZKJky9nb2oaw7rKSq2DTWRjBn9EGGq6gBxIJ+qEEFpxw1FVde+k2ESSjg2AhbNBhbiMp9chWmFOA+U8mnwMewzGVwCeKSQoa6gOhCuJGBUz3RwgKLSjMUIcgzWxYWLFqAYWOmYNeH8zDsuLOhSTSYusYDmyayuRzDZc9Tkme/7Z4nUA7GMWLkaFAHCJezaLIjf/YQgDsilORq1MZoO7j3orFoa0iiftoXYBphrF25EgveewObe6ooqUneQCSPu/obZyHVIyP7qYlSucqCAsMUxkuOiyINPTjHNbwoJiEeCXInlBeNvc1D5JpHuCXjMU4JyJ0GAz6efEnMeLVSQoqN3kSmUsLEfzsa377pTuhOCTppi60AoBK7Keqi7nivwfzVy8Pcyq1YRMo/XRGBt6qsK3bHzNC1ePHRB2BrJRSLZWzftBWG5GDNqtVYvGQRfnv3HQgHZNx5xywUCmVGNz6/yoorehApRVM0BFkl1EZUyqFUyHuwZlxR0dPXD003MWXiSLz69F3Mi4TDBGlpWJs324wcgilKYm4XEIsuXMOlTb9h/TpMm3bEQWUVNg4XzRGxJMnuPClbwm33PI61e3X0pwfAzs6h62di9as3oXX8VEi+ZlRI8OEesme4jPZchOIZJn3mFKTWbt0KL5eL3K//leHWlvj4er36++87FhtjgJVi5Dn27e6AIUnoyVXQmymhL51Dpmqhq68Cw5U4EsQhsqohGcEDt/07Jg9vwd63lwArt8Ha1wt/XueezwANOKeD9lE+R80lshj9SkO8KJ+iIrwfMGmjBP2QkwnIflUoelQHKs2Goo9kDJFTj4D/xEkw+srYsHktwnWjsP69VzDpnEsZFnq5G60NeW+PiRWmT9vDwux5q/Hemk1oGzGKFUgEjRSfYDC9uVre2tJikkMIeIbbmELd1BNg6mFs/PhjLHhvDnamHfRVfUKcDgOP3HwjPvnLVlRKVGKzWMNt2SROFwNzPWUWXUSv3jxy5EhUCrlBgTvls94xm6YYek5N/HpViOdlVTjPaJTywypSdcnBUgV1Ek09ZxLmrpiD9dv3Y8n2PiarPJKJ2dqaAfRetBUbuGYSBXEQg/ppsSJkFKyTdpveX/rjA7D1Mk+szAwMoKOrk88zFg6jpS4KSyvil7fP4rtJ0GtRbu85K1p3ym+pU4rgMR0Hiyeo1cF1oMQ/6DbQl0nD0B185/Kv4hfXfpMHG0YOMdx8ITvUEfQvDJfSD683t9Z+PMOlVk8aLEc5r20pePiZv2Lemg4eAqFTSc5S0NIUxBtPXoPh40+GLIdRztH7esMlxFBFRnsui+8FDe/9/p8Z7uyHrnXIQ9BG4EWVVOzZdwCmRcJuDbmygWLFRJpu79GZRbEsBpEFVBUTxw7HCw/fgX1Pv4ny3xahmVhTy4JORjkIwQTsYxKopuOfvCNdZN44rs5YnKSASsK7C29Kt5fgMpSiwnfTv+HTrn6EfQ4yMw5D+7r1GDZlBhNUVCIgppE2vUZif53GwIioxqUMy0KuVMHb7y+FJgW4XzUQDKNAYgYSRih+FsE7sg+qTBuUDIhezcZvvzkWTfVRNE05EbZUh/WrV2DJe+8gmQihLpnk3tipRx2PHSvzyO2qwqLSEOU5VCs1RR5JkNbP6guX3TVNtLQ0CSTh2Oxo+JYo7JldNVu5xHJH2uRapcxaZuqljYSo3kjGX0HbyGZRBnFhV3B4ECt2LcTuvQfwzpo96Ncs+AjNhEOIRxJC8caQkGCP28pI8kFXqebVK72OILIjFnCwkIPKLQ6CqowXH3mAO2b6+vtQyOYRjkaQyWZQLlcxpq0J+YF2/OK2X0ORKbISchDQnPy2SlDf7+e/p3Wn1ITOn3N5cuZUEqJJoLaEvv40qo6DR2b9BF8+7Rh2eMGggMrMHtLAwkKW0wbBJAvz8FhxL+p58s9ao6WrSyiSrg8TU44Kw67wbO47H/or2vsr2LW/B5aj8nD1S75yLG7/0SmoG3MG5+Ua1W9twfyzU3RJtiFmXPSY/1cPdqo1TvJfTcPwXoMj7mtkuG4uyPS17EOpoqE/W4AkB1Ck5vqSxl0fNB7m48274TgBtKYCeOflx7Duhvswav2AgIPEvhEb546uZKke3cbD1aSqzpDQgVQ7NNWQ8z2X5fS8E0FKEmnwybh9v2yQkoRqQxSNc+7GppN/BPX2i4Axw5Hfvxtm8yguVYjiuchnaCN4zdqstWV9LDD71ddw5umn8t0HaPRJKOjjMo1m0R0GDOzsSGPSxAmY++EaaHKUZr3jwUsnobkuiuYpJ8FEEhvWrMSKRfMR9pNEzo94LIkTjzsHi17cDVu3eRC7ZwB0dwOumxKB4U7tp6maw0eMEPCONrM7eYGcZ5SYZWKp3aFq3NRNqYJOUjtKFQzWLVO0bWigCRWWmG9EghFqUE/5YLSZWL1yKd5euA4b9w3wZPdwUMW3vnwKlrz7Ks784pfwyYEBZKsO9FAYCo0gqelh5fUSN1Pi82eGlCWJVHqTEPH78Owf7uc17unpYeecLxTQ1d2Nhx55BM/+6VHk+vbhF7feCdumqZQElwNsUrTfAm5XD527lyKwcMaVzYpyM017BPr6M5xivf7sA5h8+HCXlRe3BiGWm4cdVopC6+TCYxaqHHrLm8EykyjveA9voiRBd3pNmvl1oL0X9z35Jj7d14dcmaoT1J0r49kHvoPTTjwCgYYpMGhyC6Eq13Dp9Qi91g49F4TgP5eDatllrmbUPudz8tpDI7f0/KzLxSBb1iJTKUblG2gRPCYIoWkmjwwp6TqyeQ37enqQyxmY/dxDwOLVCPz5A5gEAWkEDTUp0NhN13N7hjsoYXNv6ET9jjwS1VXI0KoMlYAczjW5W4T6GrmGKYkB5pA5V4r+6UbseOlNZHr7EPjFldi//D00nXAW3yFALIjDBundqMzzvASVaNPdcsvPccIJx2PSpMPF/Ct/kEtgsWgQYWJ/HQV2tYiySZMdbGanT5/Wgrpk3DXcBDas+Qhrli/CivXb4Jg6vnPxZbD3R5DeJ6Zc8M3PPPUPRXSXLaVxK4Q+6urrheCdWt34njlDk0VMQ0MoFEChkEddHT1PRBVTozUTs7CIzIKkI5GMIOgXih+WDdo+FJw8Wk9qwfxF89DbX8Vjf5mHlrY6nHPSDMx56SWG64c3xlDvDyHZ1gC1uQmfFVR8mqEZxUIn7m0URkS0nu45UeHMr0i47gdX47ipdFcGEz09vdi1ZzdHm/vuvZcVXS8/+yTSvfvwy9tmQYy1IqcllHVkoH6/mJfNyIxHBymMSLgk5DLZPAbVtJGjMo9s4aN5LyEcIsmoGBzvGS7fQ6laEvk3BQ33TgS1UY73xb8wXO6G4vsECRRChjd37hK8OG8j9nVmeFwxlaLojhMfzv4ZRh52JJxQGyoDNClTnINXU6Zq7v8Xw33lge+x4Yq8hXprxaym3nQO5SqVJGQUylWkswXIaoA1t+OGjcANV16GjsvvR7RiQyGFC3kaunuBIyLloMzLrft5bCVtANq4NLOYWU0yWpe1pIgkanOiBhbwk5TSHSlDdxzg+wYpSI9MYuLDt2Ddt29F7398Ax2fzMek2LoysAAAIABJREFUf7uKo43nyUhKRyIQik7UIUQRi2vQEnDnXb9DV15HXVMTR8CGRAz18SCSYYVvp0JN33UN9UiFowjTqBufgekTGpGIh9B8xMmw7QQ2rluDNSsXY9G6nShYPjzz61ux7m/dKBXLyJDTc7tQ2Ou7JVkel2LbSKXqWHBBtURyWNyd5IjeUxHZ6H44VdTVpcRgM3dig2hXFvmqblSQSoTgUwzWM5N6jYYDyLaN3lIZU86fgtmvv4RSuYx0sYot6z/D5s072KHQrVbaImGMTcV4cuaxXzoV7819F62NIxBuGY0NPT1or1AUUOD4ZKh0fUg3yt1TfvzsB5cj6VMwceokVj319vUxYqVzpTbNx558Cj+/+QYM9O3HnXfcC10n0YmQ/nksNZ83OW5XhEIbn/6eBBqeSILSpnK1yudAfMmmxX/lu2IQt1JL4hBTTQ0G5JQFiVMjruD+X1doUSv+rY24js2pCDsPEn0YOq6//XGs20OTN0WLKBXkaDTQ/Jd+hpbDz2SupjxAY3CH6rfEy/C0i0Nu3FVLDR+EAtzIKhx3zQG5XWMC4g9pGWoHWEh/++1VDrfEmeT5qa7mZ8Pt6s1y5KAhbDQXuT+b45IPlQN+c/vt2HjHn9DywU6YpHnlOaokCxNpB99gxKt7eY3i3GcpciVSp4joKHILL+IO1hm5Id5AmObluvI3rrdS2YRQgQ00Ln4YC069CvPVAdjTG3Hh1TdCc6EdvTcZiSB/dJEHsXqI2GMHn2zYiuf/PhfR+ibEUg2CuabJiQrBOIdvSiXRBShloCgmjhnbgu9fdBbqUjE0H3ESbDuJjevXYM2Kxfh0XzdOO/NsNJfqkN6pIJ8roFwSrX2skHLvS8T5tmEgHokxk025aTIZ5+dwq5/bZsdyTa2M+oY6Lp2EgwICewIVT95I+W00TPet0aD6RcSgzRcJBtGRLmL6t6bjuRcfxrixI3HLLb+FZft5YgjladFQGHU+H844+WjUtdRjf1c7OnbvQ8L2s6abjC+YiOPEiy7Gg6/MQzAURdhvY1RbIy788uloqY9C8ScwbORoXlO63SfZBMP8aASf7dzNDrF/oBsPP/QIHJvu9Eh3InRvRObuUS+F4uvqTj6hurSQPorNpBni9qWQqti46G9s2AG/qLXSg9YhmyVmlyg3t7zDrYuuJfDGHyrBHZpriroveE9yDm8RJ2Pi4usfxq7OLAcOErLQq/3HFWfh6kvP4NuMUJ+uWaSJk2Ltee9SfuuKfw5ihz8naWUU+N8w3EHKuqb1mt/v5fu+6/BoSy5TUKRUeeGyuQqqVBCn4rthIpMvolQ1MXnSWJzzxTORu+Be+Gn2DhkJyfP4s3gb2k6DD8/w3FGuRDTxIGxvzpNruLzQrsaWNi+RNNQB4w2sE2NT6bYaVHpSoc76Hna/+yFy23aj9ZEfYv3WPWgdNmJwSh95cjYe8uDuhAUSB5BEngaSjB03fLB5W6ObSeUK6M6W0NWdRldfBnu7+pGvVvkeMOefNAbnHjMKsViYDde04ti2eT1Wf7gIAUfCzAvOx5IX9kIrUBsXOQshuqCITw/asMSYUjtkJBgWEZSaHywDca59i6Mi50kbNx4VZZ5KpczrRPCVmFeqkVPkoteiOzqQzFNyKpAUMaKUcmES3g+UTEyaOQVXXn0F7rj1CqSifnSmy5g7bzXmv7+SeYgff/+7aO/eyY6G4N7WjVuRCIYRsiU0NTdg5NGHY/WWTxGoH43DRzYhEbIQRBWth02H7I/yPXubxxzG150MlwYIUB6bzmQwefIkrF+/ETt3bscbc+YMGi6thefQyWF7hjuIOujKMMnmZm+OhAoNNzctHHf8EXjmtz/jyZWkba9FdMQXsO/9XxouGSbde5mOg27fSRNGv/6jPyBfpuFwpA2gY7Uw+/fX4Jijj0CgfiLKxPBXqTQ3ZLgUlYX665Ce2/+HhkuWRXeZlF598FpupKc3oy4M2lQ0y4dCfpXuuseEEzGeOuh2nHfedgc+/vHvkPz4AE8CIHtj76HSd7X26pIbjsxMH32QekbIzWjciuhYGRwOxtIzMUCO2GfOrWoWgEem0hj0ACm5AnDO/wKkyeOw91ePY/z8h7Fk3SdIJhvEAdAxU47Jt9uk+7WIIWRC8yGc1D333I+jjp6Ok086Hg11CTTWJ1FXnxDsNwlFJBkawSTLwc6dW9EYqqIhlUDLEV+Aoddh+9Z1WL1yPoaNHoV4cSz6t1aRzZdFlGe45E53cNMB8mU08pNgqjhEGv0pBAGJRIJvjE2GTvXkFN2ylG+aJoyUYCRFFoL65XKBG0AYurqN5o5ThuqTEI8HEY0m0ZfRMe3iqbjm2h/jsDFNOPfLJ6AhKSPATRVRZLJVbNu6DTv3tKOvP8tD4j7dvoenbM78ytlwAg727tmBq666ENt2tKOkUeuljVR9MyLJVoTCCVSrJkYfPpmhPbVxljWhWuKvCwUcaN+PbZs2Ycvm7dCp0lDVuT3PKyV58lIBB4dKTN6m9/gBru3aDh741TU490snoFrSWdsucnBxl4F8IS+kmO72qyV+vNzW4z4+rxxE+zYaoRo5NTU4mLt4DX7z6LvMNg8y7ABWvfwTjJh8HORwI0okc3Tfj3TbTGqR2o3aVGv6bcV+d8VGh7TmHSSo+JyWv1qozOvi1oJFxL33KjEBgzYKTwChhmQaOGawbEvcmYzIFgmJRArf/NJMtF94F2waRVozlsNWRH7JCh0XpQjqX4Wf5zKTzlnh16U3pp5Nd6KS2MjEDjJcF1MXPCUJRyx3tArDKVlCOBZGaVwbmm7/HrZf9ksc9tjN2Ez3EyIn4d48igdeGyaKxQJveu735fooMc90v9ddKJbL2L51G49E0S3SvgYgwxT3DQqqmDZlIk6ZNh5/fOJpzLrpSjQ3pDBs+inQ9Th2bN2MtauX4vwLv4Flz+xFrreEStXkcyAvLfS34jYbDPdpNCmL4l1JHzU4KIpotKZzClJUtZBKxQdrpXSlquREDZ2b3akcFKF7tsrkBN2eYZ6aaBAlgngyiFisDgMZE0dcPBnfvfpqKJKFyy69iG9mXd8Q5FG4VIMncQSlPnmN7ujXiAULluGEk0/Axg2foLuvG3FVxxdPGEN3H8KBjjzau/qRaBwPNZhAQ0MzO+ymEaPYwZKx0qhUijYEZTPpAaxe8xHynb3YuHkr3+FBqw6Vg7xI6+X0XsSla13bm0vPo3SBHvNeewwtjUGYBh2vN2mSFFNVvpuBUOQdXCUV9wcWZsOTNEXB7J8EGCStJGfgkYWPvfgPvPTOBkZF3iMOA0te+wnaJn0JUMIopbOD+mRvj5Y1ocOujbiC63DFF4ccn2e4h+qTa2G21wLLebB7D2H++qW7r+S2Pmb73JDJ0xFNaimjmh01lBNDClxwwYXofOQt1C38DDrlIq5HooM16Z633niaGsMllVmMJt7R0bu1XVG3GpoEIFg4TzNLKllvSBqJ/N082O2fpIhLA7H1VAL1L9+ODedcj8SFZ0O+9DR0D4hiOF0fJr54lAz1xgqxN9s0T3OUEY/IaGtOusSYmJ5Bf5PJVZDO5LFp41b059I4bGQb/vzim3j+nmvQ3JBE27STYZhx7NiyFeEAsGdNHunPLKRzFaJAxYA6Zkf/D2vvAaZpWV6Pn6/X6X1mK2xhC8tSpCpNECkaRIiKKGpECEaTGFvswW6MiUaNvUTUGA3EgoogVXqRXVjY3ndnd/p8vb+/65z7eWaHDf5y/f/X7/PyYnd25pvvfd/nee77Pvc5567Okfp1QoZpZ2uSNz4Bps8Uk3MkChcf9aukLcqczpcRJC0Qqa+yHdFET5eZk0s2x7GjAmPYTuFxVEY6E0Z7Wx+mcy2sfc0qvOb1b0YrKOOyV1yGJYsXorMtivZsm2h7nekU0tl2RJKdQDiLeqiGZtWECZzAMDP6LKKFHRrSzLGos9UwxvPtGtZGVgkdL3sXLlHGwJqYLUQvp8zlpnHfA/cht/sANu/cgUKDtEBGbYciO902Nyb/L2TZtQx9EOF7Mf1n+s1rvP+2byOTpjcV+eVHjMHp4czD4k9tXLYIvcPin9q4HOotzrTQ8xre8nf/iKf3GxjnX9dceDw+9u7LkV50EoJGHNVC0Y1PcYMD6EzqpkL8v9y4mmPsAUy3cXXYf++mNyriCjmjEXeViCbnzhjTh1pWCr4TkTje+JprsO3PbkK8bJpXOdITTSYSKmd892JYd9pY/lwqEhNYpAfFDyHp3xEfKv4b00Iflf2pK8DfnTSKlVqknMERRSQbw/BvPo/Hzn87mh0pLP3Jx/HQkxvQ1dNv6bDT5Jar3LhszPOhW7pNjPCpDU/h/ocfxdmnrsXKFcegr7sDwwP9yKSSqFFTWq1g4zNbUC7PYt3q1Qg18+jMJDCy9iw0Wl04sHcvGjPAhtv2oVys2jDtqi1e/g4PRrGu5QHCF+VgbOewbJBDZjyqw6RULmHB8JD8kxlRBfTxMGUJ0mxq8bLO7ci2SeqXTFEfax4NYn9HCMxwpEkL3b19mKrVsOrCU3D1tdci3hHBxZdcgHQ8joHBfoyMDGrIeCKRFuHC6249+OWf/9jOBxCrjavGIb2QQpJqPYotB1tohNpxzHHLNN6kt7dfzp78OZFMmk3kCtMoju/ELT/7DfaMTgrc1CesmyeTRSXvV2aHz/ya1QcSUmp17dEQ7vvVv2jTUoTBA8Be5jEldJ4JqaslSRDxLUBRIqVNdlxheWs9v6+aITDFz84MslHD+W+8CYVGCKEmJ/MZ+v/Aj96PJccMItK1As2CaaT5rlEHlHnRvI+4z4/99mntoLXfPT+d9z8zF63n/bA3kfNtOZJTcrOzCH3rI1dr45oEyfSbQv9cjUV9bDVo4lWvuAKJ+3eg8tXfolzhsOqWLFcIHinyOlsSF/BslksohAy9mWnpwtS4BbFlJMTWyA9nq8oeYcvpK90GF6+TrQJ/ErOdIB1wBIloEvG2BAZ+83ncdcENiNbqOOHBr+MXv74DI4sWO8M/A6c0woMR3cnnWAs+/dSTeHb7dmzYM4njj1uJbCqJamEaq5cMYO2Kxdg4VsepKwdQZe3UKGKyGGDl0gH0ZuNYuO5MlMpJjO+dwYENeezeMIoarVnrAaanJ+eQZInznVuFZ+yQaMD0K0GATTrcCBrNGrq6utTKKJeL6t+ypBDKzxS/0cTM9AxGFow4ZRFRaLPaoVuj2mkRWoXS2qaB3v4+NDmlYVEPPvrJT2Dk2AGcfuaLsHb1Wov4PDCj1NqagyafA58/a+tcLq9NRET/0NbfIlKn/WkYyWQW1GLICxsxHJyOonvxaeju61Imtn379rk+KNfR4Z2PoDM+gV0Hm/i3798ubWpUm9D0snq2nPLoDmXeE3HfSXF06LsypGhcAN2CgR784gc3CYPpbOtA1fX9mYTRUZIZCEOB5y2bx7IbSSLFljNadwHK00l9nCFH2Ud6thbOvOp9qJEp1YqK/94KSnjsJ+/HwjUnI5TsQok+TgoqvOfmeOqHVv/fNq5tWPutz0Odj/r70a0h/71+MAFLE23cud5SyBrkmprt5nmSh3rM4mNwxZVXYfMVNyFxMI9yhDR3jdIzxY53p3cnmZQ1gdmhhOsEYQIEZAxxwyLkRNQEpqxtxF6ZqXNss1oqaVHba0G5+Yg0c1GlYmkk2xPo/eVn8ftXvxvZyRyO/f4HsTcGlDkpQJC86TvpFkG1E69ndO927N+9C3fe9RDOOvN0TWmgFLGcJjlhDdKNaTQD0h3LSKbiKFcpK2vg0FQZq5f0oTsTxcDKU/DcxlkUt7eQH6/g8MEpcGod20iVWlHSMtb+vB7W5MpmXJSx4VQ0SuNwZx5CQAeBKKlDGGHJ260jJZaYWfLQRYGqIbUbdMDVEI4Ekglq0gLR5gR7rsyLqiDvOdTfiX2FGRSbdSxdvQixBEn8hkgbG8oOQLHaHNWO6b1F2zqmp6dQ3H8vx32pHKBgX44VkhE20azk0X7shagkB+R8snXrVr0v21FMmw/veACHJ2Zw2gWvwdo1qzA4vEBYSaRhJRmvSxFOuAPlfkckfWSzsa7l8+PUP94bfvZjFmVRJZ+8JQs/A/doMkh2XIuHc1VMOO7XeqWEajGvsqXZpJj9+fFPQWWeoES2SS7D2bx9N66/6WaUajzsSSwKY2Aggd999Xr0rXopmmHSHE24ImN4d//oejL/PV8o4v6/2Li8Z3KO/M7HrtHG1eZl6sshRw1LPfggOX/0pLUnYnVyBOUP3IwCpVPhEKpEbclJ5hnujjAPIvHWZhNJoau68X6AsenEjEUTtsl4Qu2YsGmh+ka5a09pELmrizgtLm5NegNzsuj+wXtx/zv+CalDU0i94XzEr3gJDu4dg1YbT0oynypFjO7biX079+LB+x/FqaefiGUjWVSaKUw1ouiMtHDuRWcgGy9jyzM7EImnFfXa0hFUa0ChWcIdm7vwjj8/C0G1iR2PHEZ9KoI8J9FXgWKpigpBiQCoFHJz4BRjgJElzMmCC1GqKkaXaEz96I62jO6B0HUnvZODR7lk8j2SUFJ0Z3JSSNrjCHmvIx0nfZAHBAkSvCf8piqGhxei54xj8ehdz6J/ZSfifWkkmeqKceVSSPc8dLAgsFm3bEXVyzg0MYG9G+9DWyyHRCyJRNJ46VznTOtJ8avUm+heeQFqsS75aG3e+Chy4/tQL09r0PSrX38jhkaOweiuWVSmSqiXWwgaYSTCSQcSATVmbeQ/Wx9HBxEPEpZcYs0xatJ1UzOrbAazZYYE/VxfWzArwTb+n7RrJ1GMRhBLcqRpCBEePHTWFFehhuLMKAq5GTRKBi6RgJXiemlGNIPqi9/5OW69Z7MkmUrqQ3Vc/bK1+Id3X4u2hSehUamgXLaNKwsn53c2f+OKduvCuaXE89qj7utHR1wf/Y+Oxv77+F+uHw6RV6bCGtejwwTD6bzATgM3pdDRRh03/PW7cfDyT6I8OmGm300OZnD6xjDlbNbw9myYGNs54pG63N6hajYo2kHjpInF4oqOCTGirKbWAcKmN6ODU13we+gvNIe+hUNoT7Uh8aXr8dQX/gPRzXvRXLcIa778Hjzw8BPIUGGEFg7v24Otz23CHb/9LS6+5CL0t8WRbx8GFq3D7c8extKggPddPIxYiDV2BZs27UGUJIZ0CskUS4YYRpaegFhyKWrUunYPIRxJINQyMrwUILocuyamv6qtXKtCaKZzYWRWIeaXAqlzkaCG2PppcyNLXTFk0yO4aOmNWaphfHQc+zbsxaFdh5CtAbVWHQnqiNlWUx+9iXC0jmUnnoCR01fhrp88hMWn9KOSILMqjUajMufQQNM1LgJ+1q7OTul9efJs27oZDzzwAFr5fThlzSJZtCayUSREkifzDPLLLlXr6Ft9EZqJbokAHrn/12gWD0jBc/3ffBj7dszi0MYZhMoxmbrFIgnEogm0Yuxx2qTCZp0m61XDNgIudIIwIsJqHXBTZ2iUJ+6xH89iYBEzKfWB4zHZBbFDwVKDmQxrYvbGs9k0SpWCEytwsmAOQbKEdGcYi45bjL5Fbdi+8THEawXEU3EBs8RrXnfjp7Fnqq55b7RbCocS+P7n3oALLngJQulhFKa54Q3V9mWcNyb0m2+OSDS3eY9syxfasEf3fefXv/77eRhQUTU+Pm4jbpkqe2dEblxGXDOlNqeGNWvWYH3bEoy/7WuohWtqEXF4JS+S6CKlefyzr5OZdoQbHIdxhMblp5dJRO6dLlwkFuLqmE1e6eE3rgqoUEh1sU/ptEVcxE1+8W3Y+NVbENm4E6GuLJbfchMeeuAJNMINHNy1HXfcdjtefNrJGBjuFEmkmBzCg6FVSCfDKI4fxKcv6EQiYY6J9InavWtSiHMknsWy1evQO7QS5UID44encHj3DMKtjJz0GXmYlgXse7vDlAswVDEBPr/Eg4douVwe7Bh1BAu2TCylo6GYvJeUOpo3NR9QNmNDuwXShKugq3UoHsbgwi4MrBxGOEjh6Z88hqlDo5oyoEjVaiLbHsPQCauAgSy23XMAx5zRi1y4hFYoiliUtaWz0E1nlG7RhJ7kiWwmo7bUX739HTjp1HUY7O3HxN6NOO+01UhlNULc/KF4knLj1uoYWncpCi2qfkJ45rHbUchN4Lrr34MdOw7gwKMB6rPMMmKIJzkegrUr3TzswOJC5zrh1AFNwZCYgCouIpos11rIZGn9a4wrDz4RByFZhPeUG5seZELwJcYgDbQmmihpsfVa1cayhO2ASkVjKNXKRvmkk2PvBE695HTM5HehNXtIffFys4lXXPtJ5Ko0g6dpQ0ssugf/691YfNwZCCIdyE9OIuxYXv9/Nu4LtYDmDvIXiMZz9S1bqAHU3hRH++sfulpjNj2STPiZtSajZritDW99/Zvx4OUfRv9YFWUO9Q0a0qgSU+OLaTLBKaKfYrQwySYfmYvQiQV4E3giakKd5CG2uAVUaSaa+RboQzohtUcWiTSL7ujkfiZcCCGRzKDna+/C/f/0HXRs2o9qGFj/u8/j0c3P4cdf/yZGFgxh7TFDWhCToTZsjS/BWGoY/ZkqTurKoK01g/VdeRndNcNRKW9K5SaaQRYrjj8NhXyAJ+7eiWY5jmSQRTJK07KyIoD/TLwU7+Mk0MWl+joI2f4IkRTRpl6sH0rFQ0pqGA0Kt4jryfY8LAlUkQ7Jr6kH7HqWjteGYpBDrDOMky9ah5n903jqJ3cp6nJywPpzTkPn8Utx/2+eQKsUQd/6djRTVHwRjmiJWcWDktzzvr5+/W4DxUr45Kc+IVLGmtXHY8XKFRgcHMTeHRtw0vJ2tCeJS8RkYkcTOtIQB9ZehUaUHtoFbHnyTrz4nAvR33ssHrh1G0JFNwhOPttpM4j39rFaNJR5RrV5D48ddqbvtBsS4VkHisz+3ARGmRQ4RhXvC1NUlnEkPtAhRL5ijYZkebzn5KdzQ+vQ9JMfKQ/NsvVWNgAwEUE9lsOLXnk8xkafQZ3jQWeKeNkNXxDhwzyom+iORXDHTz6AoZXniAtQIoAXCsReYp7N0sZrjL0HwP9oBx0ln1fsOYqk8UKRmBuVpRS/l8+N4KE32At9+X1XBfkCJVGqpFwqA4TjCbz+DdeidNcmFD/yY9RpoK1ZKnVUgiZqPI3omsHZn0ELiSgjp9ViVGjw3eYG/BJVZBokiVgY9UoVWfZ2XfQNmnWxlXSvnG8sN65O5mTK+nxOZmZ1CaV0WQz998dx719+Coldh+Vn9MiKOFrr+rBquButekH1y2TbSvyu0oMgkkF/OoorhktItKYxsmBYn5uACXW5zAZqzXYsWXkidm+ZwdaHJxEPEmKRifwgIoQNreZnNA0zU/2q3TkN3wqLqcVoy4g8ODik+lcnqrdYEXKcVirsWVSMsvTnGh4Z0kMi+urJCfwvFzEXinjg4SjqdeZGBay+cJmMCh7+7s/R1tWGkbPWItXXiQ2/26nIMnBSL0LtDVTqVZvQ4JhoKSmh2sxxolHRDCRGP1r5DAwMoVgsoVQsI9PZhf+6+WZc97oXY+FQCrGALpxllGsVLDj5GlSDMPYeOIzKxG688rLX4g8/34RosQtTM9OWlgvDOJJteDCK94MHGw8SbsDZHDnhZpFLbTP71myRzecyc+MKvHSjZmy9UOJY0+8hMkx3UOv/0kPM7GR9RFd0VvvGPLzYimPWkRho4awrTsOOZ36DbdsP4C8+/E2Hu9iOeN2lJ+Gjf/s6tC04AdViGZViSZx2yhI1b5FtR41OsbzghV5HGI82GfKFXkdvXMtgW4hHzR2T94Ke457aGvrSe66aG2wtIUsQYMGCBbjqytdg9y8fQuXzv0S4WBYPuchZIZzFE4ZQ5fkblxvS17UaHiKKoYnHaRKn9JLIKf1wqf+UCNqRwnVCBjYJ0NW53KyefM8Tle+p3J4pJ10gkiks/cO/4t4L34n2XFluE5lLlmPy5Da1UHhIFDIj2BJbiH2zUVRTKRzfHsKFg6PoiqYRontEKY96JIUo+UHNLBYvPwObN41j15MVxOnWWGPmEHIjNG3TKhJyKnqCdVtMOmSypJQ5hAJtVG7c4cEhM+d2TB2zPJUd4ZEeYxh6H24a1mVqkRklfq7eTyWSSmN57eZ6yHlABiiVG2WcdsUa/OG2u7F8aAiDJ6/AH371OIJiQkDMglM70cxQUxdIqmhtmADt2YxcHSbGJyQG2Llzp4gqmQytUt2w8loZPZ09+Mb3foBzzjoFs4f34KLzT0BAMghaGFl/NSrNAFt378FLT1+P3c/mMfF0AzFwYqD5dHNyIfvFVrMypbeFLvFFyAzQLdMiQ6wsVRb/3ffxGXG9nlrtaqeMkiFBzAQRsrVNJPRMiMlYKspWkrH1zB0zhnQ6g1yBEcs5PLoh6mwFHvfKxQjFpvDFL34B37rl0SMbNwC+/Ilr8KqLz0couxBT4xPKquZvXIFSDmT9U4L5uUkTDoQ8OuIeDUhpDbjsjbiJ16ITmCI+0NPTjdC//M3lQaVUAZdYR7oNl1x5Ffomm9j0jzcjtYXeUzU0WpYYS/3QMgd+3nKf/un0m0fnkku9NquG3ZieViMOzU+XD0fTRwlaOSKab0kxCul7mSI47ylRvTiPxonr+Tniqxah55sfwtbz3yn0mLDFeHcdnTecIiBmJ3pxqG05ikELhXoCK3szuGgxhxGTwUPheVS+WqEwD400+oaOl3vjY78aBWdV2pxdI6aoZcUSwpl4+2xCEYQaWDXjAY4rpTXr8PCw0nn6RstbqkHXCjOCZy+OAArbLpwLxDRWEr6uDkUfLbzA1CqKtGSJ1ex3mzyR2s8kIrR3pd9UuIizrj4VpYkxbNk0huJuShmt5ZJclkMrxjQ9QDbZgUjcrGjp7HF4bEKLvrszi/EDBzBLhU+oimxbO9raOtRZYLP/jxuewvihcaxYuRLReB0pjcoMsO6Cq9UJHCBIAAAgAElEQVQymZmewmknnIG7/v0pRBspgZoh9toTcYyPT6hdxA3EqMQD1RBiUwlxbXlQjwuSm4ByT4/K8qDXuhC4GTWXlgZlf+zvGwmDmYW8tJwzpt+4mk6hEbCGkZgtEbM4Z41LJls8pjWFTAtnXrMeZ7zkbOybkHjYDuJoDPd8751YftK5CIXimJmeNhFNxAziuUZZNhjZwzJB/3p+BHXdE/fPR9JkI58cDU7Nj8g+TZZE1Q20Y5kT+sxfXhqEolG8/GUXY0FXP7Z88gfIPnEAiLG9URJqR40tdYdawMT/ND7DFrTAJdUtR6RTcdbIRN48b5OFPp35aMjmUmEvPPDjNv2HZZ3X2dY+N3PFEnjrmc3d0FAU3R98ExpL+rHv+s8beMOJ6h1RhG5chkIrid80jkU51g+EGzilK44Ll9MKLySHBdY4HBAtCh5bK23HoqtrBX73H88g3ezQw+Tm8iNQdPKLJGCgiGbUOuN3Xg8JKeoNIkBfX49NDXRRmJvWxlJwIcXQ5JAzDTQzJ0GK5tnL9SMuuPDoDOIXhr/H7A8zmvO9bJxLSDY4QTSBkRd1ITWcxnP/vQNNKoYcQr/otFGEMtMAUmiGqkhEF+PAnho279yp6fW7dm1Dd3saixYtlJa6LUtKJQ/hMA6PHsbuXU+jWi5icjKHgYEBtHdmZLNZyE/jFdf8lVojy1Yci8d+uxWV3TGZqzPzSZEt1uLIy5yMGFiTGnvNi9RscBkPJj5XZmDcyOxZlwp5JNlXdb1e3Sj18zm3iOJ7+mZXnUtkTPU5D1jzFPRjVRtKhXmfaErnN69lR3Xpodkvnxu3GY7hhCuX4ovf+Ta+9u3vuh5zC7FGHU/c/gn0H3uuDO/JWOIr7twcuaY5YcOCjnWXj46e8xFiW7+OeDLPLfOFIq7/mth2kTDGxsYlmeTfOzs7ENp730+DdCaLrR/7LhKPbEfAcQrxGKLsJ7YaKIUDzX5Viurm0BKv4wf2PFOdmvOkSxoxxGkFvi/bbBmpgIQNN6uGIBYXszyC3Ga2E9R0uCKHa2atG6I9r5iPdLZj0Z1fxYOX/TXaxnKgElgT5RIxzFzei4cGT8CziVWoVetEvpCuTuLCkRZOXpxGF3unjiLHeB8JJ9C7aD0ev2MclYNEP81VkadxscjhXdY3thnABKNs4zI6yhSedjq0gG21xCUmMOLBJ14Pa15mJNzAFBkImJE1KRddWUZvZFzRelSCeicwn9u4jv5otkIhtLe1G72QJu41m3JYQA4X3XgB7v7GH/QZJUrnwh86jJ7hHrR1pBTBSRlsNCM4PHEQd999L/bu3YXwzKSM87bt34cgTAM3G6FB293ObAsz41MYXrhIRu2DA0Pyj56amsAp57wSmWQCQ0OL8Pt/30YTSW2uNGcAhSKqH3mdowcP6cASycH1bU27S+F7RAcRa1NGHn7G/OyMwCZ1J3g/2G5sNJFMWDuwWiObyyYYWDZk9Fu2lqjx1s+xBEnSe8zsivje9LYiqNTb06PNG43xWVuGw2fYd0oGQ6tH8PEPvFeHAUe9DA924UMffiO6+46XXJMHC78/6e6RDPfnlE1cVV4PfIR+8T9BJ2c4f9Sk+T/VJlJLMBwSHsHrZ7Yl7fDjb7ouaN2xUYN6a7WyNgwL+UqNIzUomaE3Ygi1SADKhllnJTvbEe7IIDLQhXR/N2Ld7Yj3dAmsaRJYODyB2uPbMPHYs8iQjsaUpUrChiBl45UKKWa/17ntuIgtNJoqHl27m+cTCSPWDKEWbtIJHCt+9yXsuv1BlP/lZ3pPotriWUeB8RdncNeZr8e2mTriLT6YCBqoacpBfnIUo1u2Ij27F6evW45Tl/Tj5DPPxvFLT8bjvxxVRKsVCTqZCwgXlmeqJOOM0uZIyDRQIzUpgo+GFTm4YJgGcwFp0gPvm4EGQq40zZ10zqgza+fw62RMvTljLFUE1nChOeWfO73JeGqoDibSq1Nehx9TXqbzYYQTCSw/rxfP/nE/GhOMygROmug8Lo+Jwqz6uByhOjDYi7vuvN/8nQHs3rMb9cIE+jvasW+sgqo2SgTFUlmeWSesGsHCRUMY6O038If65MIspmfyOO+yq7BwZBjbHx7FxA4rb1hrClGvtnRNqs3CIYwdHtN/6YU8xyHmMvfuIPPMAhltZ2dmnJrK0Gmqd/yMIf6X78FDQUZ8bnCZzdYN0CZdrY0B5YHBTUy9LjcpTfdsdpUNPVOZ4xVunU2cfc2peO97341GuagM6MY3nouVJ52JSKIbs9Mzc4eFNz7nNTbny/H0TNxIl3kg1PxRKKZ0cbFX5aOjP7qRKEfSZJskwetkn533ngc761tluRte8cYgTOJ2bxtiw4PILh5Ez4oliA/0IKDUjNGJ2A0RPBb21SKSDoXNlUuIFmuoT+UskhIFI2gz0I9IbwfC6QRq20ex7X3/itkNWxBiZCKn2QZEauNycr3YRWwhEYBxHj6+leRPoiDKTR7F4q++D5W+Lmy5+iNIShroke0AzWgNtXOX4K6zLkYykcGuXXsw1TmM3Ng4cvkKipNjQKWIanEGqWgYX3n3m3D6iSuw4fdTKB+MolTNIxqwjmqIoSKLnURC/UHR3yJEdFl32onPGoosJ95QooyVkknQBMTQSJ2UT5dS8+ustZjCsfZltO2l/pe0OWY3NTeaIx6VD5ZSMpdicuFx4xAp9TU3nRrIGKpV+VwiCHdWccqlL8J9P7wPcW3cFtqX7kI9xujSoUl3iXgffvGL2xGJBqIVHjp8CDu3P4flxx6LHXsnEGVUk79xSZ/vjJOX46KXX6CevDjfrQAHDh7G/Q8+gnf+7XuwbtUJuO+H29CohUWW4EHH961XWcuaZJGZBaOd3RPLKNQCc7OMtZHmAZK8l8YQmhE6LL02HSBr1TmXCsM/vJuGcQj4d66neCImuirza1Mr2ZA1yva4eZUdaoKCpaCMvk0iJJEAZ71hPV77xrfg6ac3IBEK8Kuffhgr1p1HiY2ki8pEvP0OiSBcz/Ook36UibKBeYPc/yTpQmCVi8BCadyGdoeBzZ6mCQM9o61t2Nvbq4MsVNz8aBAlW6reQLFZRf3gJMoHJ1A8cACNfeOo7h8HihW01YFEyShq/H5uVHoReeYo0UQ9DGkDNSQIhZ4U+j53PZLrj0PjqX3Ycd0/IL9/FNVIC9GggYBEDbGJGGEtFQ3XW9b/dRpcAiSKvuEIlvzb+1BdMoznXvV+pAnkiDUUYUmmGTitSAuVpXFEb3gdJlKduPWJLVgzMoRFmRB+eu8T6FlwHPYf3I/JqSl85f3XYXEb0DuwDA/8ZBtaxThK9QpSkagE9IV83vTBjiEjLnHDVCxWo9oCZI3KTaVIosmAPO2jQpsZidOufuMjYQuG7QsuaAJYQdMDGxYhuGjzhZy0uXygXtbGRc/+rlEnnS9XiykkQas4CuUmcuVJXPjOF+O+7z6MRDylmvxg7RFUgxksXdSD3p42pNo68atfPif8gqNhxsZpdhbg8cefRM/QYkVlCk34+fp7evHRv79RSp9GPauv0VvqmWeekoHex2/6JA7tmsahh+toxlqyzJEEjwPf8pZ1SCpaNwEBN7TfuGrvhUyJxsORm5cAH1+WxlKvTTKLlWjcvKQt8n5KJSN02uSZYvjxz37gnEa5BhpPyvfnUG/+Pg2Uc9MgmQQJT9U8ZANRYqE4ll3Sj/FaEa969RXoSSVxy83vw9IV58mMPed0wb6zwc86f+Nqs7oZODqc5m1cX+ce3bv1I9TtGv9nes2Ny2ucnc3NXXdfX5+yr9Dm5ecHbOVIhkeYnWJ02qW6KQJmim3oHm+yRyy9IZbvzVH87j+gDUI2rx660U8tG8Sx3/kAKody2Pu6j2Ls8G5EeMCQVyYbbsrd/HR2MmysnURieoI1SiSMVT/6LGYSUWy55mNIVmpiO/Fw0Oeg6RiF+OEmKovacOjCfpSDFEIa38ETNYJnn9uCVjSFBWtOxFvf8lY0y3l09XZgz7NFTGwMoU5fI9rHuBSYD51/N9UH38FNfRd7xxYlI65GPc61tawtxAdBAMWnYhQFsC4hH5cnd09Pj5kJcNE5/2iJpVyflWZxdnABhWJOp6zIGCQhubqfMct8p4FimdMRSzjzTevw8F0bER5voRkJMHBSGxBnCkneNr2CiyiVCxJS8M/ymZ6ZwMMPP4zp6SJyRdqj1rFm1XJce81VQCihNLNcsYHRBw4ewMaNTyKIxPHtr38Td/5gE2qzTWTiaYGXMqCnVRCZd26MCwlRfmqdoq7v73O4tu9E8P46je6R7kJ07h4yc+Gztt6mn8hgBxjRaCmaOKZlbjoElWZxgX6Msha5jcQhQoZYpm5Gs+u/xmMhtC1I4ZTXn4Qbr74SSxd248Z3vBEdXcv1zMj8EnCo6Y4WGXmQNI8yjffPf370nNsXR1navFAk9lHdZ1xcg7OzU4jH0+jKtiOZjeOhDbsR2jF8WsDFwyI7iETF9+RN0DR417f0fsg+AglPcnUSf5YEhQa9drxDvktd+MsF3bdCKHTEseTXn0e9Auy+9K8xeviAicrZD9aUPWvUk3qmjciNQWL1QD/W/eJzmNl6CLuv/wLitYrSdvPCptmtsd/VjkED09kQUu86G/UgpgiIUAxVEtejcRy/9hSk27tQD0Kq45YvW4E7b96K+rTV2easT1vXqk1m10gQWr2S8eVsNx1pnAuIG6pSKllaywdaqwosUvrbNO9gno6U4VGXq9qLM3Gdo6GiJ9tjIrAcsUTlkEaf1hnQktT9MGGPmyCvU9oECoVKE7VyE8klUQwtH8LuB3cp/Rs+sQu1cFnti6Y40lZ/hee57BNTqFTLeOLxpzA6ehjFagV/dtnL0dffi3yRQ9PIC45q3vETTzyBZ595Gu/54AfQmx7G5jundEBX8iWNDNXcqGQK+ZzNOubhVGYpxSgqK16boKgxqxK0WNRUNtM0b2hLr4lC26FuYF3UKLbOHI4/M3dYzpPqcREoisfCstvl2iJmIMojPcyc95g8qmWfaxE3FqO6KowgHcZLr3sR/ur6t+Kay0/C6eddgFC8R1MayKbSQeHUVUqx2XP+Xzau750fqV2PpMPzI7A/sOan4irTaPlTt4O8Fs3gKz/bhOem2xDaNHgqoTlBRIlsB0qFgknOPKWRBueudmWNZrpdLmZyROviuYrVMs9Amy0Spot68eTl/ygY7+/C8t98AWP3/hG7bviUhOPynvDDmIhcq94Io0p0dvkCnHvLv2L/rQ+h+PF/l5skHwQfojG0WmjwwYQ5cc82SzEWIPb3F6LElhRqKAchdLZ1Y/W6U6SxTCTbtFAr1Tz6+hbh3u8fkvsEGUnarLG4alAeUlxk0sSSxVUlFdQWAaMDCRMiELgDTO0Od9AZsmuTzRmpIhGjdJL4bv5E5NUSfY45uR0JCXa7VHuFjcBgabeBLKI8ztu4/s/8mVKtiaCWwN7pvXjVuy7DAzffJx/g933hvWhGK1h3/Hq85JyX4OSTT9Z8XSL3/sXowc1pw78bGlxGOI9Dy1PpNswWZlDO0ySgomvJFwt43TWvxUO37kYwDkSSEURaURwYPYS2bFYHmEdguVa4cf3MIhkpcGJfqaxaX1lZk1pic7rgywM//C8jJn+n7oNvB2p2kaXUtnkt+2HGxAjY0c5h6GYazx6hGG0uvfZsNNswFvG1sUI1RIMkamHgnL9Yjb+4/m34zHsvxaKVZ6IepDA9NeUAR9u4foC6aLn/y8Y9OgL7++5/99Eb2m9cHlgqMXj9AL720434Y24QEwViDTWENnSvD7hYSMNTTUKrlFodcaF2lk54l3XeALoh8KbJPqMVCBVVGu34lJ5v6rWJfuSmasBICIX1S7Hi5n/Aczd+Hodu+TXyTdZIDeRCdfSduRb1YwZQ6+7A488+g4995gvY/a1fIvjOb1AVS8Z8/MyTwOSE9Le1ifI6JTR4KvyBl6EQM08rpn46rYMYCvkiDk1MIZuK4uVXvgm18Qx2PEI9px1EPIHN59ec9326It6sSBhmcs62j48MjOp+M9shZK6MjIRcpNygpBiydh0c7AOtVkj+kEWN7HCNtxximeKmETACcWAZWxeK6AS6KN+LeajyiIsgf54G5PVGAuNTo7jk7efgnlseIrUNn/n+J1Co0eOZEc0irmcrEcEmJ3jJ0iVYuHARli9bhsULF6BaLQlA7O/tRyrbrnp/cuIQanXWcFAv94Tlp+Cem59BiCNA3QAvZmjjY5OqBz2SzoyIf9dBzpTWfXylxUqpbRN6Cx4PXGktsiSRQZo1ctm+4cNXhBb32owN+bM8ZEkHnNMtN41ooXZT3AlmJK90UdNlhp5Qw94+sZZWDDj9qlX47V0/x0vWZDCw7Cz16GlGJyKEk/ERSfb8ZIa8uZcfseMMAvzX5+t0j96oL7Rx+TZJSr8QxbPbD+PLv9qHg6UU8jVzRVHb8I+dJwRMdRX2nfu+indnpanUSu/uepmIIJPNGlDA044pjecoz/NAtjEgNj6YPTW9PxUiyRjav3gjMievw8NnvgWPlHZiwaWnIL16BPlwHcVcXS4Df/6612Pff9yN2uf+U35INqjKUqRQJCTnQHF3xY6x/IDyLk4wr73ueNSWdYKGKV6Zw0lqXALcSATCzv+za3H3Tw8gyMclVayWbVwJf4f5TBs1T3B8rarygWkw02PtAvV0G+q/8iESoCIyLKoneboBLWksarK9RNUKwaVyqaJoEwoZ19lHEppwC+yS2VxNhAfxo5kFxNkHroi6d2Riu/GfmU6VK1Xkck1Um02cdtVabNu0HcXDOdz6wI+Rr+VQKZeM3FAqKWJUa7w2ShkbqDWcOL7JSGtYBqmHf3nD27Dm+HW4+977VAotPfYY/e41x6/GjgcmUdlPIs6RXj5XSblECx8TSIgHnEza3x1ZXlMYnTCeRAulwSIYmK2PbWKTryl1pl0OBRoaMm1kH2mUE2wT2SHEDIxAIidDSPDh3Vy43pzxAIejKdWUHJCoNYOSbXrNIpYIhusqitXnD6N9aQaNyWfQ1rcMM7PUWFuGoo2rWUMmO7RQcaTv4109ZBTgkGGTeBpngRf4pxDmuU3OSEvmYTyKJ3fN4gu37sXBSgwtMtmcvluQ8PaFZwWMND6q+NrBi9z5ht7T2Gh3JiDgQiUB2tP0vCujTjFnJcn3ogiBvFoxkfhQIiGMpcM47tF/x6Z//B5a/U3kO6pItqLIizAODCxchf7+lRg97+0oRo1iGW858MrdFCmSeFNIkVTeaF5SzWYY+XOHUDttRHVdXIO9OHzZmvH8fyiUwDkXvwl33rwPKQTIF4l90EW/rtYF6zRuRn9PRHiI2Exg1V8y8HKDoV3tleXh1zCvLhFTGk2UikWBeb29PYoYrOt40wnvc96Q0mKJ1MMInCkY0de2bHqu9mUNyujMdJuR0JcgfjI8a+RymbOKmogk4lh85iDqrQp2PrkFO2Y2YqY8Nec6yefC66rUawJcKGzIFUwEoXSTwFzdOgepWBRtnV3YuWePWKvMXLhhHnv8Gdx/8xNIVJJoeHsescZ4qIZxaPSwFrgGeCkVNbYcRRfqx8aYFpcRi9hnkRjdWeYSwPOkHgM2LYVmfcznpvqVLUNHVmHtx03d092tDMhHRf4uvg8R7UJxRlGaNa7MDqoVYRlkonET8XdywwUtHrpJBL0VvPQNZ6M8sQHRZI8GmvGpqU3lNq7cT53BocwU3ctvXPVyj+xEy1r9YID5fV+vTXcBT+HRIcy/uHsnbn4iQEnG+mSlMYjYgAAZL2wbeXHg3eOPuOVTQGH8WHvNS0c1IdMkYr4RLsBhvumzZqtyFoy1dhjFuAnsQ4WM/H3Tteh62ZnYeONNKFzcp5lFjN5M+84470o89fpPILNv3JRGfGj6PHZqeU2vlTimnOAG4FZmWlw8phOhN58oK1JuFt5QZhNEYnlyvejsl6JcGMT2PxTN/5h80ybrIjvVuFisbLAHZEJzoKOjXRuP9SgXjBBOhwXIM+lIJiu6H/9dM1c5ST6bUdpGDrT3VmK0tihqtbOJEoBEzJm/sw/sFwWBnWZFogePQPvnUy5xQTY1d7htcRrDJw/juTufRiW7Xy6PRO+pKOLi5rUVCXhUqjqomLlYthVgZnpWYBrTwzotgFjr03OMNXCliVe97rV4yxvejg237tF9YMuDP2eZSRy52YIimqmOSDYxm12+uEnpq81SRBvQtXh4nxhd5C3teq8G2BkPXNarLlJZL5jP1MQwjMw017Nsy4wX5jJAx0BjqcFnxfKEG5iqI6HDySPOjmxTMbKr5xxUcfHfnI1qbidCkTjGxsYUxeNzRg4hOVZKoupagnMbd95UvheqYedHWz9EfW7Xa5hACPFwGN+77Snc9kwUJXCOFdc3cRG2FNxUBQavrSNn6dbyhPSsD90cpgNucpolzs4lj7rGpM1Z8SkB0zVK9bzJHL/XR27eXJmTs8XkjOi44Gb6M1h255fx5Gs+htClAyjEq6iXa4hnO7B2/YXYd8nfafFYP4yxVMN7TT/nUi6lzrx9Gi1CtQijRhOz/XGk30V+KQ8Ja5moppRWs4WXvuqNePiX46iNRWWA3ar7mTVO9+lGPnpvZAm7nY2qiFBCZ+0UjbvBZb5u44LgK5+flSKFBwY/G+1R6FAoET1PcEZS0hmDBhJxo8vxACToVasWHUHAeGWemM90sVIqggB0nGCca6fUG4xGtpFqyQrOuvoMPPZfD6PRvR+hSF2icrW2NPLTDiOPX9Dojv9GJL3WYFupLHF9IV9GKpm2A7FZx8x0Hh/9zKex94kyigfokUUFFrMB6/tycRFDkClIKIR8IW/SPi1u1pwcVGZaaoJ/Att0CDclJ/REFAMIY2JK8XkzQs6NJ5GayGYpMVK3yd6HaqmW2H5ztq1UshWZ4em3S3lktrgGRumQndNEM7BwwqOVNASeTvzzY5HoqKGSm7H+c5j4gqXJfLFuFxg5X1MrEc6RfXIk4DqXEx8C5xE25iv8WFLSNfPff70Bv34mjCJsrcTTZNORLWYZpR8eF9rYc3LA09AMoW0atxA3OeVruzqswT4A00XaWTINlOxOobuFbJL2KO6CONfU1QDeBI4nlOxbHMLXjAJDt34K9VAE93zpn5Bbau917LK16GyNYPz6T6AZNXI6HfbpRuBPLA9iPH/jUulBW506RqNVjHz6KiGkRCzllhCn1I0E+G6ccM6rcdf3n0a4FEFZg7isxmIbQ3QyotsyzQtEVGA08MwZ/hvfkwudJzSjH69JIojACAdMq9mOYOQiP1nc23QCcQIsLomSGUA0JtCKKCgpkh2dBnoFjaqzuXFSSXGlWQ5w1CZnzNuEO3+qRyIJ1BsRFMoVVCJlnH/92bjn+3cjMjCGZst41Hx/z77hVEU9Zc5oKpbVj6a/FFF7L7tT31JZQFP0R0ocb3j33+H+bz+HUDMhk3v2Ejgnie/L665UicQbWMfsoVwqI+nQdT4rblzrf8esNUPVUlsG5ZpxwnkPueG5oNva2sWA8tRTH42pIGrvaDO+tiR7jpghpxRuSOvTckPzuUh258zluL6Zdstt05Vclm14bjTvdxQDZ2Sx7JQFGN21RQe06vK4Hch8sa999MbVWpy3Keei8FEDwPxmt5T3iKVxKBTDfRt24yt3TKPcjCOIJBFTOUXTQmarRGts6IAyjyc7Tgj4ZppNE2f9YD001miG+pl3lOeYdrV3GE3Mp8H+w1Ijqj4oVTd2sZ4RI6GAH1btEDf++8xZK7HiK3+Pu6+4EUuvO0tCx2imE7nxMCbe83lw5LIALtYMtGadP/xXd8YAGlvUNiqF59JMpIWRz74GuSb1oLSBsUHJBHrWvvjlKE6lsfn3OQdImSRLvGOe2hHblKQ5cm4Q74e1dBghOZg6JldFLgJ+tpT4sG6siJvVyo3O+iuRsJaHShlXm8TiVtsxE/HaXKavRHipWJLXstg/bqj2PMCPN7ZWLStdZtS39w6bfVCLA5lt0PXZf/ki/P4/7kHQNqrIrFlznE3sRlkq13QvZlpGBpkHqBCwcUbiPGBKhSLOvOQyFEaTGHsir5q3QsM0URxJj6yq1ODGK+TN5ZKbiuQNuqIoGsq5xMAskUkCAmt2MDPSsW8tRZUiY0htHbqtGLBjBgV8ETnmNbJONiMCo5YqC3LtNJ/t6WASVdM2LJ+HodUWea1OBcLRiLILcYJCYWSHozjpVauxZ9vGudrUYwsqoZy5ok3Pc/fS9+vm7qwLe0fVtM9Ll2WPQ8JTA+OFMt7/9WcwjTY0YmnZvsaTaStnahzknVLGJC44p2Q81XWiM0Q3obv6Zx0dRn9zhm1EgxkxbWK32/FuQfkPwtOUp6IMy3kCayMwzXKsK9/2IJWP/rlM26IxDD/0Zez53I8w/qP/Rq1Vw8hrX4bCypWY/dBXbFzHESbY8yKubrxQYEvNvCkbb2YhEmDBh16J8SS9mDlBwMjvTCXPufw63HXzZgTTxkGm7pSfm6AUr52pNFMjfj91yjwRGAUZOVWXiLFF83i2j5pIa7KCcZe5CZi+8cAiwkzrVxMb2CEoml7UDjQtGNIDqUHVbCACfexvhpFgy0N1HdNJ+zPbavx3Rnv2q9lOESOI1y7taBLleoB6pYYX33g6fvuT2xFvnxQophaPi/TKkhzZRC09j37O+R3bBvYHN593pqcPp5/zMjz2090ojfMwS2rDMjctFug6QbUUyRpGCzWBe0g4yMThMRC447rm16391ZKUL58v6B5ZKm12M6xV+Tv5M1QCMRvgvWPKOtA/oFRZ6bHsd6lAMvDR9RVMyOEGirFNVMznRBflIVcu0zzO+uG85zyQxZVWORZGPEWqaAiteBHnv/VM7N35lK7DJKVO/0uket7oy/llpGM8Wp463+rC39v/8XWKM0KoBjV86N/uw9ZiP0LRhCyBSBhiek5ar9cQM4Mayi8AACAASURBVHD4/n7o8bbj3dawMYEecu8d6AOn2NFipCWWiKUTNr3MwJP5LA/Pu+SHZiriN7hpR63Z7Qd8MdqwtmLU7vmPD6KeTmP3pe9CuVZE6sozkDjxJBz84JcYQp8XZeenygIH3M2xtMXqRG6uYqiF2DUnAauHEYmF0ag1JIfqX3wshpedgSd+fACVotVdOmxicbUU+F9+RhqU8XSjAIK1kjX8WYvGEecM4ahNQVdLQYivqYh4f7gQWA8z/ybwwtm1mjQrX2PycMNSCvH3UnjPeyiuc5P6XLaEmggHpmG1iGoRhx+CRAmZYmtUhqWkXLg8kCKRpAzDOe7mhNevxR2/vAPDi8M4dOggkhzWrXLAMhih2O6/RsQ3FFbAm1hJtBgy2ilbOC+5/Br88ZcbkKkM4sCBQ2g1w2hv78DefYY4c/FyNhDbJpp84eieau3EEyLaGE/btMncJnK6cACWrF8jvNcFpBJsz9nmdbOrVfszI1HpIVDpyNgSUj0ZIFLCFpyxvxu0RrklLXA9+433T6YG6qNz/ZgjBwk/as0RJ6HzZrSC8647DQf2PWMjXnTY2cYV8eN5UfVIXfv/eePyXYMWfnH/JvzwwQaq4QSiqR5UmUlyJAoZhRHXVmU22QwELioDfaxjrVJlnbIOWPC6UD5cwuWkM1LELP4ua0K3YTwyxp8X7d59nYIFRh72Dr1PkC1A9z38PhEammicuwpL/u0juP/E1yA8PYP0Jacifcm52P6OTyFBL2JWdPOr+KNSETvdDF22YhySHx5a2YYlbz5P/s+ZNDWsJZxz+TV4/M5DKOyIiNHj60RNkBdgI4K247Ia+ql6goAK5XrqmyaRlIuE/TsF1lwwMioLM12kqZqRBIRiFktO0sfNwe9rU8bBk7PWrGGQ/Vqi8qRxOiYQf5cxpgi6HfldHVk7OOXCILsX6wmrhaLISxQ6jBUvX4oHHn8M0ehhbRIt+LR5J/u02DOUGHXmUNu6SRB5bcl4Gs2ghjMuvgxTO8vIbyG63kJxhuBVXiwpjprMF8qoVQmaMOMwcYGuwx0MJP9zo9EZhP1gblBD43nomEujPzQUTWS1aoZwJflzWUTm/3VfWTK5mUMei2C05+EkVRVxAL2HqYy4BvnyrC2NQdGAbluLyniSJlAnZkGhCbW/p752Ncan96NSG0cmQ8TbXprV67IXre0/6Xrxv6fKvE/8/X/9z/dgMjKCZrwDkWQbYikzDPC8eR0YPBQ5z6vsNOKPd/iIy2fmhNw6fY1Lyovv6+5BoViw2oSppXcnEDrqDMtdW0ZjMmUGzlMsKtXR3CnvLt4saQI0edGpOIbv/Fds+dx3Ubz5NjRWLkD7e6/F1jd/CMkghBjra3kWz+uXebraUTWv5ztXwsD+jhqOed8VCBJhJIMoIp1dOPn0V+DJ2yaRHy2iWm0iN5szBNNZXwpwopF7vaE2BFsE8xk87GfrnrA/rAFeBHNo5Ba3dNctBuMTOyvSRl1ZC9s+BFvk1FGyOpAiek5akPqFcj5FWRN80J2SiziRosVOzSRt/JqrRTV9SYveAT5kXcFqxkUvGcFMq4idW+7X93PR0ZXCz/eZnx7z+0WcbzblgMHPxgxgejaHk847D6F6Gvv/MIFIPSHTuVYthG3bdittbYU4gnQXopGEEHxrCxGoi9mfmeaqN0y9ctLRLW0DMt0XAUL6VcMMZLimdLklVNk2vVFRBeD5WtlpWg1INEsfIueWNFgLju8ld01xvK1lqM3A9l7NLHI8QhuX8ZuNFCEQ19HWg0Uv7kX7ghRmcns1cdIfEqZimseWcp9Fh59b38+PyPbF+dkp/+4Pt3/+3u/w0P5O1OMdCGe6EEtl5iZ88B1Z2xPxVgChgUOFf28h9Ejb6sDXUX7jGo/TtTvicaGfczYf9L2RiMAr+e1jegIGHwSlbGYcHAicmGs/zAOoGEWJTIrc/433IGhPYsuV78Z0q4Ghb30Qm1/3fqTnNi51u4xiBkZoRIpP1d1dkvLPAQTVoIWpZB0LPvpq1Dl1oQJc8qa34rHf70NuWwSVnOmCebLu3LVThT+nnIvW6HymvDO9IZRUBxlARy4uox2vV6AK7T7TSUOsUwkdxroHHIfpwA5mLGQv8exhROSIjwUjI4rKjIZKT1kvp5lq07mBdTEPPJYTbIdERCAgiOFVWWzHqD+udkkY8XQalQp7vTUMnDSEjmP68Mh9P7FIQ9Sb7RWX9YjcMEdpZWpL8zue8lb/cqEsWbUG/YvW4sDt21GpxFDImWEdSRbbtuxCe0eHShOiypOTMwIAdUjI8tV6+Hz+smGlY4WqbE9RJJLvNhR7Ww4f4PuzfGCqPDw0JE41gSebD2TPXGmrR9ndIC0Dy1ivRtDRYS0i9qNVwpDdRkxBLUT7/VxG1YoRghTN5VkFHTSck8T+P4arOOeqc7Bj15M24REUY3BihVbakbxv3sb1KPH8+bj+G5+/ce2zTE7n8defvRulbC+iySHEO3oQTqTkq+XZWsQseD28JyySWDaICPpY+1pRoYSMuk3ATcpThjeSi4kDovUglJPbtxmiduSliepO4cHL8ubbjFKsaZliqLZxvUfJ+Pyg31ecjp4Pvhlbz34rytN5xL/0Djx04ycxVA+QDMJymHy+K8SR3+3TPP9J9LCCAGORBvrf83IUExFc+sYbsWdzGeV9wPjeaZRmK4riTDX52fI5yt2sXzjf8Iv9OuPb1sQlNufAqA4RXn+jWlebhwuMt49kACO/N5Ei4YLvx1kvmixvaHKj2kBnZ7tmACnFdQtSelJuQIrtOTLDeQlzCh+7SBwh4iWbirp8RhRjiBLJGpqzY81Ct2tJB5acuxz33v4ztLdnMDY+qgXPQ0GIrwO1rN6k+39R94F1KOvyxWuPx4LFq7Htrl2IluOoV62VNDtDA3Nayc6qFqQgpFLiPNy8XE7URZiHgTDWx2XH49a72kQlJFPcyA6s0wRHZiFFHXgExej04QeS0xHD/L8ccUezhoydxmyF7SYjuqS12AlAGYWXkk6T+lk5ZWNMxCngoPZy3oz2SfaAlYTm11xGOJpANZHDy996MXbu24QIsQcX/US6cIezJknOYz/N7YZ5GamPrnPMKR7dQQQ1FPH+z96CHaXFaKQ7kWrrRiKTpZWh8ebFt7Y51fy83LBSvIt33kLo0bY1AReAPoAmk5nxFT8db4D6qM7sjQuGkUX1kRM4z31YZ6XJn+F8VR8RWf36ekfpgbtQcoz5+/igC11JLL//G/jjyW9BtJxD+IPX4OEf/QLdG3chQ1mRU8b4lMPD/fNTEJ+O8waRZjlD5PDqM3HBh/8WhcMRjG2tojLZwNRYDqV8WVRJ/n5DM9lTY9O+qEXNjapF5IyxCckTxWUNZKQLDgbjTB2SPuhRZaATWxncAOIic8GyHUGgq16FbFZLrHfTKBbzyGTpF30kjWMPkveG70WKKP/Mz9Pf34NKuYAoxeHsSTtpmmHJHnCiEiYudlS2pxvVSBVrL1+Lu371X2gFRW1wwzCIskfmNq5q2WTWMopwBFXW4/1DOP3sl2HTHc8iXWhHhZMWNfeX0+Zz+r6JiRkd7FR9FQrcPBmMTdA10iOwbuCb0n5D7bmB1FJEQ77RJPHMIa+thq6V6DyRaNXicqkwxp0FFjusxQtw3lwUshcLeSxZskQOHbn8rNJrk05yE9YklhH45gCtufQcRkll1pRMpw055gFCgCybQTKdwLpXrEQtWUJuclxRzrO45rfT5kfU+evyhTa0slRRJFvYO1HEez/3e+RTvYi0DyLe3ql7yhGyxEq4z3h4kdg0V5p6A0K2g7Rx5/UhFcHCIWRSWecAAelpmRtKl8qr89P0XJTWLRU5w/yAaChmG5eGcZY2zQey3BGoTaCaJhxC/+PfxrPv+ypCv38Q1QtPRLBgEDs//210BMa+YVrpU/T5ULscMlzNoNRHtUqA0fY0rnz4R5gd48jIJqpTZRTzDVQKNREt1CYi4lksoFY1hJu12dT0jOor1U6OTEHqHxegro3v3wo0c4c3lRan/ABsu5ClxZ9tb8/KwzebSqPM6X01MxqjQKEldhI5zDVkM6aCUZSNmhOEDkeqfep1ETJo2VKv0nM4g0hg/VF7mWeT6JMNglQsTyJo6+1BEAuw6IIleOD3t6NQ2Kvszpz3HVVQLRhLr8jt5ufN53JoBlG89MqrsfvRPQgOhjXcKyAWI+8t/r4wxsYPC9hjxC2WCxJ412stkNQhOicJDorkloILMkuQfEJDd0YOpsI1lUk84HhPNc5FKbbp0KSskh1QXFHUDhbbuEqXiTxLFM9B3swSOJmPkZTCBJI76PJovWndI9fnV8bnhpyTK82+uRhbLtXUNQZN9A72IhXN4GB4B172hguxY8dmtBzpQp/BaafnJZxzSL3/2p/auBHSGMMVvOPDP8b+6hCa9NNuX8j+lAbhRTkyJWjo+UsUYnwoHboq4R3fPPTH7vU2rc/3TENAxk2Q583wqiBvVmBpsOtpsYaRhzKRX9azCVQd2VunrzyUjzT2+TVvS6NI7m1IEKDntn/C7L5RTNzwj5g5pgMj734z7r/qnWgTTzo8x31W9J6nyODpJ80sca5mCJF4EqUVwzjz11/FzLZZjG2rojhdQatCTjLmVEBs4NuDYl1IrS3TVqKGxtFmCspNw542U2qe7qxPeRdZs1k5HUYg72SysxpAqIae3m7r04aZ7jRRnM2jUa3pfYylY4boXNyVUh4dnR2OWM8WEAEu1q0G5hABZcRhFGcqVy1NC+Biaklmm998rMslzaRRWob0wRgGTxnC/smD2L3lXsR4T0oF0fz0DIRZmFhE7k9BIMLDqRdcgsl9VcxunEWrGUWjbtkXgSd+D+8Jx2hOTZLOmEalYdI5sqyYqXhnR16bZ+MxSjEFZ9sm7GprRdGgrpqfhndsLdFjir+D2YznePv2ju/zsg7394UKNQKWTCWJzAqoi1prrZgnSYTtS5YxBMmsDWb9X6uVNamwRc6xMayYXbFXnMok0dPXp2wzlIwhtSyEodX92P3cs3P7lHdlPt1RmZ+TnM7fzD4jnL+ZqRLPlRt404duRS3eA3QNIdnVg1DELHk1b5qqrXIVFWpxnTrPPMiNjCRA74mudQFbPV5/amSAiJBQf8IJineWH1IJemDDzWxlOpJmisOer+PB+hPHD13yOb5aTc7RXmCJJHlNRD/yJvS84hxsPfU6zCYaiH36emy89kNoZ/3BZhPbDO4OzHfNI9fYUENu8Dj63/QqLP/oDRj940HMHGihNhMgny+JylatmBsDwThGByMNkAVNdJgLs67emYjqqseddIw31AEDAnpkpm10vHTMFod6oFHjMGeyaU2J54FWzOWRcgQNtUGcn5babBznQXJHMinU2ZBGigxicswgiKWSLmILktTPUiWPVMKQZ1uMRkLhwoln0sj29yGZaUMuMYv+lSPY8OCdKBbH0Qz53nDY+pVCV9kXjqKrqw+9CxdjyYqTsfv2XWiWIqg2WC4YEBONxJUm+tJm755RFIs1AWIqNajGd3Wn6WTtsOZPa+qiy6zI4ZKsjiUH6+NqUbUpD1HyibWhdIBSxGLiDF8CMZVmr5UgV1+fs/LhweOnHaCltptlFWzVmeWrMees9UPChge4uI6Z+VCEQracX/8dnW3ydeYG6h4YQD40gzXnL8Xk7CgK+cIc3/7/tkGP/rf5GSIPi4/+8y+x8XAK9WQPIv1LkcykEAlbf5sBgPpgkZ44MJ3llLMx9k4hyoofyq4ShMyaw99Unpysz+RqSEcEWY2YKsdL/GxhM4Pmmc3hTil9wdtk2oNjjLf+rU9plULzEHCT+PRQww1UXnseFr7rWmw++TpUQhXkPvQa7P7YN9Cey6MrnJS21r/mQBqCBOoXEqKOY/1Nf4vsay/B3sf3ojya4GhTFKermnvKVJAkAfZR9dlbgU1g1xhMmyJYoZdVJGY6Wk0WbJlxma7bXAVlqeMWgozO6GZYMmolPaVYLDdaDSTTUd2PGGvuitVpOvwcOV2gX5MAldH9eAncHOSB9/Z029eUHpqti6w6xVclH7hoKiHH8GKKzjIm3dmOZFc3IskUplqTWH/Zi3HPz25FMxhFHeYVrc3EfrUDClMZaqtDuOBVV+K5329FZDYjsnyrboohEVuoruKCcnYt+/eNoVZpIXC8YJYUHELNtJb9XRJY2BbiRbOG5DPnPeW0Pt4n8pmjHGdDQbyTQpoai5pgI2NISJBg5DYLVqbevF4OaWPrTAIQaZ15z00QQw6zhAt0Z9H9s/6nJ7wwhbbpBWZFxI3MDS4mnzNnZ4eAJ0b/YD8yvR3ItrdjOnQIa89dhmc3bTK85ihgdn5Enb9Jj3z9SHmTL5bxtg//GuVIFxrt3Yhr4yYRallbj59NGAvLDreRVWaaBGpOlRb6Q/a4INwMxHAhsVtjDtwbWI/NHDD8KardzsqFUdgJ23lj2K8VgVxjJU1+NHcRrhnvEWBGT5uT6njGYaD4kuNwzD++BxvOeBsirQam3/NK7PjBr5B+bqeIGElK4o8iYjDZI8OnFo7good/jOnuXow9th+NQ6y/6qiWKJCvKYKZyDqEsbEJRa9MOotcPj/3wLiwGFIqdSpSDBDwNa2RFdiftHTQj4vkwZRxSKoiIiN5g86FIRQqeWRSSU0baDW4cAsiVGh4meprHoYG8vFwjEu5VENXV4csVxhdpL7yWYbIB25iBA3Q6JkrMQhTRANguob65bEc72hDvlnB6kvXY+NtT2K29hRKTdO+MrJwceZzeRNJhBN48aWXYXpvE9UdVQTNxBwrjNnXxMQEUumskUTC5B/PYuzwLGZmiA6b+6OymCjdUdiSMqSejDMePJRCclPQ7jYSbpj3kxsKRyIE570QFGP7i71vWcs6yx4Oqg61YqiRvNHeISdPKqlIE7RgYmUSnxXpq+0d7Sa0JzPKbQCapPMmcrPz655oowO71ZS5O1Vb/LuZEpSwZOlSSnWQ6uhCRz9/bx1d6yJIdWawc9s2M2dwr/nkIGPwuTrd1aN8fja0PYZGqIgf3vIAfnrfNFqJbqB/EVLd/WrFeYop12mZg+LqbJkRvTVWm2+1WXkUIHR/emVAhDTLiMkERpvP0dJc7UtChbXx3UtpGsGKQBFCFDU5CtjPqz/riezzkGRFXg/Pe8E9iRocYbl8GMM//gSeeek7kZ7OI3fNOXh28yZEf/MQkty41CTOO+l4AfT7zQ8P4OX3fg+VYgj7Nk6iORtFpWhuG6V8UXUaWU2cK0qQibYoBw4cUF0Vo4Y0n3N0RAOomkEIuTxTKBNu8/uJ9Eqe6MoA7h9S74g2p2nQzUhCgCkW0UR2kQUoJ1R0toOPQAgb/7EwXS+Y1vMmEtU1twdyFbt7ekVW4Mb21EDWfOLSSs3N1LAJpZxBzTjBXIAuemZ7OpFqzyLd04uZWhHHvXw1Nv12B3YfvgfhjPVVjW5qjDA+i1K+hD+77u147padCNdZY7PGZAlhdZw43rwCN1FgapKSvxomxvOIOg8ylVQsr9wi05S5OMdC5uSzxfvOdg9TwGQyjmicQ62LaO+JINsRR7wjBLb+YwkbyOXBrWqJnOwQ8lNljO8sIKjE0ZHtEoLPZ8MsTx5ebl3E4sYnlxJKHHlnbyNKI0UiVuMqnachBANGMT+nhOOa4ubPtmUR5yjObArJ9iw62zqwv7ATJ1+4FvtG96FW4oxae70Qq0+HrV+rag2xjRpDNWjgmnd+C7nwIKJdi5AYWoBwOmsB0GU0co7kYcyfbzAzkPRBb2dSTPtz6IHscUFc7o5E6szIWoOU1OwmeZ6nnvOfFVDBm2FvQhTZ80WYemiPUq6mVMcTrT04xVPyyER6r93VCcULWzSIgdv/BU9e8T50Pr0XB4fbUb7qRdj7ia+jB3EkXQtANiNKm0KIrT4WZ932PUwcmsL45gaCfBPl2QIKlQC1EoEd1l8t0TW5mJg+8b/9/f3Yv3+/wCC2BKjh9QcNPYRmczZwWYR1Z9BNhNTYYIZa8qWay5P9pQnmQC/WYmHQrpbkCD4QuTbWyygUaPNZ0MZRKhgmAk35Wgr93YP6XUoJo9bP5f3V/ReHmMWujafsaqerZkk6WRrmqSInMb+nC+muNqS6ejFZnMGqy1Zj6x2j2Hv4IbSSs4rMSiFpuCePYfkE4pVvvAEbfrgD0RBrSBJcmMITLDGmGK1x1Gar1zE6SmF5HHkSMlxfWCm02xCGYVgLkJuQBxZ/doajRUJVdPSEcPJpK1FJHha6ykgd1JnCsuZnVmStOLskO5RIl6zWSggV4sjtD9CcjSPCodk6LA2TMRqkyfr4u3mdbKsxS+Kf5UDikHhGZ6EWnK5YKQv152Zgq4n3PNOWVV86mY0h0zOIbNaR/kca6Fnajp2bDagSc3deFjg/w5y/cWkvzOf0wB934rPffhiNRA/ifcuRHBxBjPOZKXap1hR1fe+WtbtIR9q4NvpGskQCoXzuj7avkVmcB0Y09pD/88Zc3MBC4MypkOCTX9BJkbINJZ1Le90i8uGdC1hfcj1Hf1IJn3Xu7GFuhs4khv7wTTz7l19A4vd/RK09jpn3X46n3vFxLAyldcqKG8rFhhbazj8DZ9z8BRx8egwz2zn2gkSHGiqFskgObF2w1tKUPFqQcpaNc+XgZzAksSUHP8q0eFp7WRcjhTX46WVsKhf2CT0QRP6sjdZk7WtqE25GpuIkSgTNKtCsYHziIA6P7UGrSVqj8Y45aEwAl0tvfUrOKMrabu2q1Wgj9Y0T72KMTsyE3Oneagjt5M8kOduoMEOSI6wCJEDZj0gmgUxnP6ZLU1j1yrV47rY9KNXHsO3QHxRJGPHiSeqAC+aK2DaIc/7s1dj0o902uM1EgIhFDeXkM5+cnhJnmKf9nl0HEQRR1fUc68Lv8SojXwpR2ULQJxRuoZDLo9IoAdESzrp0MULxCkplTp8iDdR5kSkS2ybTjB+3YjSF0bVodM81qK1FwB6TW8qY3E2ZZVqZUyxpkxRMKBHRKBJbm6wbmyIwZNNJJ6yvzE1SUKrfqAgk0+cPWujs7taG5AbOdLQj2dmGTCqB8doMjjt7IZ579hmNnqFAgPZItomPjI19XmboWqHEC97+ke9hX6EDQXYAyZ5FSPQPWztP9jQ2zbBJphRH68kS2Ea3KrJz/zmaqOZXsR1kIdhefuMaN9hFUaalHIdAXqy4x4Ta06hpSp27za6O9Tm+P32YJvq2j1hNDlnVUe+yb6J6QTqKkYe/i22fuxn43h1oRAIU3nkp7rvpC1gUTyJFCy1ukgBof+mZOONHn8eWJ/ZgZnMIyHMKm03N0wgWWo06ckc6lTErFkYFprqMUAJ7rN/IBzo9M6u0j0R9LhS5J4gDTEvVrDY9oTZTvxiSy0WnVlmIJQIwPT0htLRWmcGh0e2oVui95LW6jkTChe7wAuPz2n2XKknjWCxapBMJ9HR0YXhgELFIco622Nne7iRm9pQ4lDpUr6LJD9BsoWfBEOIEOtJZlFHGsouPx7Zf7UEQrmDz4TvcLFoqT0Jq+fF6lq04ESPL1uPZn+zQac5+bCQes7k/DsvgY+JG172aLiJoRjE9My0JGg8btnr881YrTBGdhJUois0pLF2TwfAxMc3z5UahAGV2pqCNSnosQTmLKMYFsJ1gA+CYYfH9GX0kDuB8JqWTAcLVAPs2ziJR7UciltIJyufFSMu0XVkUsQoZHJCBZsoqK/NsM7PmJ/PMwDSzE+7o7tThlU6l0N7TrZSZh108nUF8pIH24Qx2bNtCtficc+XcBvKbeN4XeKgWKlW89m/+E610F0Idi9A2tBiRjB3CygxbTdkJMftgYOLn8BvX6lsCwQZe6faQq+zLUAJGXLB82QLz99CRLxh9CdK4ERGs0bRx/ffN5w97JZDoeTbvVfWFK+C5AX1KxHQp2p5G3wPfxN5v/BzVL94ix4vZl6/HQw/ei+HRKYFT5PDGertx0dO3Ye+zh3DgAQ6RLsn9QRPxOHCMzm9y5LNeq6HFjIaOteX+K3MA+hvXaihQuscSAUynTaxsfWabycpFxZRKG52nvqNqEgCxYV4VFArTGJvcjlxuDNFoSbUsDztzEfRAHVHmhA4Wk8+ZWJ7fx9Tf92WZsnGLE7Q5cc16dLZ3akGypJnjG3OiTSyCSiEn21ue0D0jQ4gmE8j29qIYKmHx+Wvx3M93Ip2O49GdP3KsI0r1HJMpaOHMcy5Ftd6OQ/dMqHXDe0ItrMBHaYCr+p1cXASYcrkKWk2OSikgqhLESP1il7l5wXx/orV9I0n0rS6jgSI48jrOrENItKWEPH4YSTWyhemiq+FMRWZtMHlVsf1IYwORNzjIyonvqWEsAwefmUayMoz2bLvUXRp/wllURLSdeICfrVLMI8t+OAUJ1G0X8m58qm1c/wwSqaTKF9a7HD+aaMugb3gQyXQbirEpLFzfh63btiFoENC0XNmDt3PRd97GpQ/yb+7agH+9dRciqXbEB1Yh0z+MkMa2WgYrT2sGQpJeqBSThxZXvG1UlbH+0OFvZTvI/1IPHPmNqwPI1Vi+t0nXRAIc6q85frLjSgoplkcuh/w5SF/hqNFU2id82zevmQp4PW2oiURPL3oe+Bq2f/6HCH3ndpHQ92YD5M9YhsKtv0M2mkAmlMBFj/wE5e5hPPGzLajnaa5dUCQ1T+SQasbZmVn93YvGreHvMwNbENq4nMlKI+1GQ/pgO+VN86g00bHImKKz7ufi1YPhYGMuxXACjWYVk9NPY+GiCvbtGsXE5AxCQVI/y2nsJHZQKKD3axmaHo8yRbQ+qWxjqVt1Nj38rASkGOXVKmsEOH7ZSiweWYQ0hQCKGrZYWKuaTM1cR9p7u0V5pMKkGqth6QUnYNOtO1VH7pq5DQ06BfIwSiScD1OAi175emx+chTl7UzVLavhYiLoM3/zkp9D5PHRVAAAIABJREFUp4tcvozpmYLmB0UTJikUGUGWrNaLrdfLGDwmgcXHN1DWfbU+Kj8r2WNjhw/bHF5NKgirPqbeli/2a/nypQzfmwyzYjGnTcwoqbajyjP6UYeQL06hsD2EcKFPw9nZzlLa67jEnhxRyuc0nEwRu1EXXTKdsdGnxFlY5tS5bqIxOW0wE+jq7UE8k0I004FkNoV0RxI9x0Yx1SphanTP/x5xRROu4/K3/Qtq6aVItfUjGFyJNg6n1oFYM3koe7bMwOTNZg40Kj/dxtWh7sBiZbX3pldwjTk5mZ8DyzEVBjSJ5jh34+tIsX5xUZmb0TNSlKI69UlEnEurYUXgTiT1gVpMK72W11EndVqFm4iuWobBX/4znv2LTwH3PcUGHKZTLTSuvxjPfeZrGEAaS//i1Vj7ib/Dk7dtRTCW0DhGtgE98drX2uS8au4YUVPnhC/k1dXjBKV4itPxr8wp8tU6pmdmdMKSlEEiBvusTBvVxxRbxaKELTQ+3Aha9SriqZ1YsaaKeKgs6h37wKGA9izk+LaQmy0hXwyjVGggN0NeM5HmrJwWuAClG43aOErdC01+sPmxjBocaBbUW1i3fDWWjyxR+nZk0XOBh1Auzmozd/b3ItPdhRBTxUQDx1y43m3cKLaP/xahFIeQtaHWIEhnM3hect4VeO7RA2jujaDJFoizH6J4wlM+2XfloUX/KY7YlKkc6/95jCRiEDxsuB76FkcwuLLGjrMOAx70Skk1k7Y213vl/UxzfKfAIS/xc5xkN8VQ3YNoTBY86hfX6PVF0X1Rm61RrqERaaKVr2F8WxmpSj/SiXYdJH4kjieAsF7kpA4uPTL8GPm5cYlTELASPiFyjQFz6jzEY4hlUkhmOhGKhdHe3YtwZx4DJyzBto1PooEjE+xfqIfLzz86lsd1H/4ZWul+pDv60eo7Fl19vXNBguWD8AWJC1gyEFU2uazfuPwzywWBpAQA78uulJ28UkOnqVV6Ic8hywS0eF2Pljas6sM6cMk0kVxczieJKhcOfXL0LEYTpteqsWWK5rpg82xpIpEWkte+Ah0fuR5bTrsBsckZ2ZYcStTQ9o4r8PSnv4W2/n5c9eB/YirfwrbfjKFUrDvU1lJu/39t4oYhyXxgU5OTc5pbXrCoi06ozfEOpUpF/5eLgxBiM8uWVlOEdZvDyptpaDqtJAJUC3n0DBzE4iWHETTZNqmiPduN2Rxnu9L6xc+9iciZQumO0iCgVongyae24YktE+hsa8dLTlyNZokzm2i6xkyag5pJajBTOKLe0SCMM9Ycj4V9i0w8r/voiKxNa+/0DPQi2dWJVjSO1EAWg2eswDP/tVXSuP2FB5FvHNbnIPGgs7NLm/HMc67Apkf3IThI5NSyFAlF3JgSHrTcdIVCWQdaqVzTxuXfE1kDznjYJZIRTZUbGGlH/6pZBGSOEbRzNjOkKNKOtlgqOWNyox1y7dAi1jIih54T4XXmdj4bJGupq6vXlVvUKhtphob/nH/M2c5BuYXn7plAX2IREsk04gn1H8xtRAcmMDs95TjMpgcmWMcNzWyBXtcCKmNUxaXNtYMlA3vA2XYh1vE0dbMVLH/pWmx9+hm0wjalns4f86eRKKMTs7CFH/33g7j5rr2IJPsQ6xpEZuEKRElEqVudTR67zBVZvzpCkApW9YCspFBP33GWVXrdk12hjWtOFRSJ/x+q3gPMrqu6Hl/39f5m3vTRSBo1ywXZwtjGTVRjU0LiNIwJoYQQev0IBPhB4pAAST4IhCRAICEGG+OAMTYG3LtwwZZlW12W1aWRps+83u7/W2ufM9J/SD5Lo5n37rv3nH32XnvttawuYA3qT1pfixKV5cnqeZpsAfFLBAUCGX70jyAP0y0BWnEBWiJza7jawAcV2g4Uy+Qy6PvJlxA95wzsO/c96NRrKHebmE220HzF2Xj8jofwzs99Hqs+/Pu494YtyNX7MDs7pw+biLnUx2kVMT3Se1OKRKLYRn7n5vMsMNZJfAisfSkOzrqWI3yk+Rlf2EV/vpajPXo2D0+JRm0RgwOzGF9zXAymUqlPXrOdjk1+kDRP1Jd9S35e0tZMo7gpggGnkaq1Lr76P7fLKPwL73kjwghPd05MBRpW57V+/8e/QaXDnzcw7LLz1uOVZ12OgfQqaRTziymjSc+GIm+k+0uIZ3JIjuTQf8F67PjZDkXo/TObUQmPazGTkNKhtWqng0tfcw32PnMCtQP0ljWmE+vpxWpZ78kFz40eCeKYmpxVKsnsl6OQQeKUAiiJGcm+EGs3NrH2jHORTvVgenIOM9PWDuLaq5TLOn0LhTwGBtNohgsoV2cwuzCrYQRpKVMhgzy5bohMIq9WDlUvyN6SxxXLB9jAvjIWyQpZfcxUONpI4sAjMxgsrUSUcEKXabOVaKJHkuBQLUuQ3VRKzKmDLadMljW7lUNMlWXyJVO5KFJ5km8515xGN9LES996AXY+fQiRxFEzaydV8zRzavKyaVVCpdA/ec830UivQyw3gMTYOErLlqPO9daoqw2kCTKK2JGYQvqoJl7dUEVomIuxELl5Q2sx3ptbp0F6r92rGOXsG22HGVDlGSB2ctqN0Hcdw8hrTqmWc/Uv0zqefhKdc8HBc3XjolDyRnYQFNNYvvVGnHx6D+p/9i/oBB3Mtqs4HJRR789joieNq/78/TjzbZfh7m9tRzxizBzJvTruLxehGDzauB0QgeVJQRYUjckYnZleefkWP0RAqp4AKfYrG3WlRwYYtKVswd83MXduFPZ7O4iHc1ix5llE0EQ0QdkTU/zgzK6BUVZfhQTMmm2107woPE+raDqOaBjB577xE8SSSfzNu9+IpCiR5nNDKR3K3PzXzQ/iZNnsTshsu+jMcVx+znqMJS9AKk5dq1Ou6gzHHCLPDfUjwtq6P4mxTedh283b1O88PP8kZhp7RSM0CZ60FEAuedU1OLm/hoW9DDIEEdPiSUsxkzTMas3UBVtdTE/Noc2gU29ogJ7WQZzJjSXjuPT1L8OhF4+jPksYihmWTU3RGZDrSzpRBAqlwUzP4yi6USKolA3i4DiF4aLI9sVR6Ith2fgAqpjHwuKsergMoDZ6xwzOQDrvGJmnxGu9hlatgVwhg+fv3QtMZpDL5Di6b0olmkIyjyDOR3uZGxmQU5FycUGzy9zArMN9y04kf6LfuV75KEXjSTSjLVzy5xfj2YePoTA4gw4WbUjFtW6k5qF6NIqp+Rr+/JM/ALJrECn2Iz++FsXSICo10i0bQpLbbI+xdFFj2IzePFCJjuEztq6szmVPOLgnty5coiJSBcBN4jDdtU3vZ0g4V2cu8s4T04mWmdQIh925tOUMHolqlItvQJ6a+LkEMVwqJL6zHNhMiLozWMTIk9dj5ye+iZ5fP6M0bbZdw57OLCbjHWz86/dhaPnZOOOq83D3N7aj2XQ2iWpSGynd6kPjLbMm40YyTSiL0kJK2bedm1OdSAofa7I6c9MuKZI1JNNpjeNR0VHAgUAvOy1JqjCSxjxWLt+FZHIRrWYUuQFOA+WRTGfUP83mehFNZJBO9yr7Y13IMRi6tFcX64ghjliGtWRELCe2ctKdBTQW66g1FlCj189iGeW5OTzy9Db85I57ZF7Nh3nhmWfhsgsGUWyvwmB0tdH+2Hohw0Ynbg9S/b2Ip3KIDHHjvhTP/OgZtUcOzG5GkJmS1jQRWva42dIbHH05BkqrcODRE5qMKZV6dA/lseRmUHkP58sV1KpNVBumQ3zixKRQ+J6+IkZGR9BpdhGViiUXgpOl5TnRNXcBtZpEYjGt4yRdHUSMoLyNjYAyZaSSf5tjXKxDmzU0W1W9ZrY/iUIpg9JwEYt1utVzGiqJeres0oIpIu1EQ2pDLwZ46vbnMZQeRoQqjqfRD2WiJu451TaJ6prtjQbVSUmNccyx4MYKTRObP5BKskWk0I1OsovL330pnvjVIQyt6CJIT9n6s/PMiSMAnWaI791wF25+YBJBbgSx/mXoXbNGrSt2MiSNxIyGpZqo2wTbDFOSzahcPKxzQ5SZ2YLkkZg2/ya7Zmke11tlcjNQVd3zkvnJhXKx9RM3JQZtZweoKBrQfyhktGVLKYZcYMPm/B0Spjkpw8hlBlDOe1cnfQTtP7gMy771Gex52ftQoNdqq4WZTh1PN6YwE29g0yc/jGUbLsbKS1fhl998TqmkSahyTtY2rPVBjXLJZj5JFFww4lG7vi3THqV+buHyz3wYhOHpm0OgiictR/AUDNhCaNYQTSSNjJEJcfErVmLjRSvQbLOma+PAzqOYmSrbYqi2kE1R7yiKsGISI2wruGdvi4Slgzxnjb8svnA0wCInVeJAIhUjrVW2KDz5Vm8cR74/jlvuuBVbH30c73zrJrTngebBBPoLg0orOxq/o0VKEem+HgSJNFKrchi79GXYcv2zmk+eaD6GVnDSdMUEfzHA0cN3A8654GXY9ZvDGgDoKZEKSjc9Iu3W+uKpu0jt5BA4Mb2ogMfxPhp0jwwPq1TyShNauM4ki382BcdT+timEMLRSJOo1dQPMRCJCLS1WHUSaR6Vvd6YNhb1t6xWZX/TCctziAANRBIN5IeyGH/JEJK9EWQzaWx7bCdmtkxLWYLXRsCS7cLFhXkro2j1kiDLy/qlTFs54pchcpzJ6DPJc8qpXcTjedWstVYL+WVZXPSWS/HgzduxfLwH0b6jStm9bKtknniX2028/69/gD3TRQT5fsRH1mBo9Rqx3yQWWG/pXspbOogiSnIJcxAe2Jovpv2qqZ3QOoeaYzLvZqr8y8IaJnYGOBnp1eRZ+IA9nN4JDWRgFKTjHFUfqFPbpfdMW4oTnF2MDfSojxjtzaEQTSI9U0P6yDzyQQyZ0Oh8nJYRYubSbTbc+3/+VUSWj2HqlZ9Eu07fmTbqQRf3Vo/gZLyOc173Rlz+rvdiYMMI7v72riUShyhyTppVrCanC8XZUpLjBbjJb9a0hfiBiWJyQc7PmbcP6WgLC2XUm019Dr4IEWcutlazo9bJ+o0rcOEr12Pn9p0oT7YR1uyz8D6xnrUpIPZR3KA2g0eap7YRWtjvkxwz+7BqrDMTIbhmmQNH+iIa/TObDNZiXMwiM3YB8owi2QbGNyzD6PIUtu16DJV9DfQ0ep1nr0V61qaF/l40IlEsu3gtCmeuxrM3PC/q4Ynm4+jEp0BCCjdmtVpXxJ+e6cNVV/8+nr99vzIgyu+QX8xgJuRW3NgoFqpVIcknpucwMXEC685YJy0yotAqExRALYAQPPNkeNaf/BmpX4hsQH0rcortz7JpbZtesNZFp6PhD9OHMoUSOfYRXHIqFaT8MSgzh0uojWYHB9dUPbKAtRcMoHdlEQ/+zz0oZcfUZ1YJ1+miTMlcotSSCWIJY4rTTJ954kZiEW1czUDnrBwR6huhxnGAMBrFqgvHsebyjbj/hucwtiqD9OgJE7d3Jy7/w4EI+m9d8bb/RCs9jGh+AMnlZ2B0fBUqi2VNSzUrJA41jeevxUv2FGm6DFIdySJHui1RfMlhR9vLP3UR/CK3WuCU1Afk0yrPQWkKS1ep00a920UlaGO2WUMtao6g6jG5FpDVwaxnzDE9xqFrJz/C18h0I0hH4lgWy6IYSyIZOFUL1obpOMa2/xQnvvsrdL95q8TXNHoWAPdWD+FgtIqRM8/FH//Dl5AYyuOB/96j9IqRh5uL1iCGIFvN42VkZeLklPK5eQhQsX7jKcs2kLxuKhW1fCq1hhBlL1zOh8yNhxTw2qsuw/TCNKYOLjDJVeZgGAAtNHgfTLGQIgIqDQJrpnMhSfxM8q4mvcLvg4GuZSNyGgM0QREbCm93kJdReFe1T1xjbUSYOYETWtssE2LVOT1Ysb4f9/74HqzIjZpCIqCZ6Gwhg0RPH0YuW43U6Bieuv5ZpHIJzGIrgtSihvQjEdaslvJue66B93z0A3jy5h1OEzpts8Ed6kIvuuujvUkTEycn8cKBg1i5YqUc8lhSeN66XxPcnDa4buqNavE6FwquBbLYGJj5/IxH3LTZU4eV6BmmUkpdGWDJ95ZAmsdV2I5r2SY2qVQ+AzMm1ymnLKmJVryG5WeMYt+2HcjHU8jSYocGZa0mUlQa0VohN7uDRq2KTIZa14biExPgNTAQcu1Qj4xkmVQui3YnwDmvX4++1Wvw4I+fx/CqNJKDxxCJkmtl+lpm1cryMYZXX/t9hJkCYoUR5FavR09pQCCdKaOw5SeKn+mVc+M252XIztOWtX/A8kLpLenGxD4I7gYIbi2sNQKGEdzEveTGSQdxVBp1nIw2MUPurWmfIqmFazrKS9QqH2nc3KoYGC4lJkZtNa21g3JNYFVhAL2kqEUjSF16NoZ/+E/YecF7UVqwi+XTboQdPFQ/jF1hGcNr1uOaf/4yOuk0nrzloBucj6lWJW1Pin6sq2NuAH1m1lJXV/96aRJ+wkq1opOWNR75rVTTr1IeRsyVhtQQudHGx1cglyfnloPzMRmDeWCNlpj8ko4SaXpk/lDGhkqGFDjPZMXSkayqZFFtgJs1HE87vo6EzCUI7mw2Q0OOBYRJQTIuphI/n5/AIkKpzglqaIV1XPGnL8Hdt9yJlclRbf54NonSYB/i2SLGXn0m2ukinrphO4r9GXQKL6IRmTUiP/2EZNbVwCN3H8Sn/uFzeOymbSLJcAHnC1nmfTpxzUY1wHylhv0HDyFTKKK/t+TorhD/WYEukXQaWoH0vCxAsGb0AweGigpEdKZfAozcZJml1bwvMZlUe4cBgWP8+SXdaYNdrP3H2VjzI+Z1erBK/K92oB5rM9bC8rF+zJ84jqBu4JQyApVPtJupoZDPaprLanCzRhFTjWoc7CqEXeTTBcxUaMaWxiV/fj7CRAFb7ziEvtUpBPn9CAPTuxaCrtMTuOmOh/Hft02ikyogPbgCpTVnIBZJSGmDa4EIcocEmnaIUqKMT73zYmr4c1uIl0ywkyi2tTg7CIRykx4bR/BTlypbBW99pHYsgulWAye7RBQ7iMaZf5skqRBChzKfcuezgWu/kUm+9kg0R/y0yZkO8KO5k3ptugcr0j1YdtPfIXbeRhy76MMA7SzYL2XWGQUerR3B0+0ZpHoG8Bf//m9IFHvx9O0HNMequpbNcg0RGMVNoEcyKVcCetMI/HLWi0x/+Vl403jaNSnG5cTOadZEA2NTKAReuvFcRWIbAneKjhyyd2OJGtVzXGcJBzBLIXc28JaTMQRqBcXkfMfIzmvU5FWbC8ycFzhL7IcvpGLoSAeLTu+Zi1kpu9LqhkYBqeIhPayQChJlXPGOjXjqV5tR7GaQySbQt2wZYqkcVl25AdVYBntvPwwkO8itnEGQqinCN+pmvcF0+ZYfPo5PfflvsPmGbTqJiEzLoiNus7tSWIwncOjYBKZn57Fs2YgWNFVPSLThBhKRIpdRqqzhCfnzWFamckQePmyFcTCCxAn2N40vzp4xNyazHdmZuhYjf1dOeU6CVTI2ak2ZionNDTEUOxkl9z4aLHAcAa/X3ApaGD9zGXZvfwb9qbTKGvZ3tWkLBQ0MMIMiw4knLj8D8QKtd7WDOFAQQQsxNLvAa95/GbY/fxRzuwMMrouind4nK1jvrMjnVq038fYP/ztmo+uVJqfHxjG4Yo0OPa4JAlKScquW8fl3vQwvG+uIO9Fg6h62lIFxuJ7bivxslQPEyEnw4b/dnFsZ8g9cSBwYrkZDrHvbZYitHdQbzE9NY37vFMon5zF/YgadahOpTgTRkG5trCtNbiTmoHBrHDGNNOULJsWqCEnlokwITYRZR4YBlmUKeN2ztyGaKeLkBR+20SaiZ4yo0QDPYhr3LRxGJJnDO772TQysW4Hf/uQFq6NkMs0hAecWHo8rdSNowt6t6k+mZE7xgBtcZPZWG1XJmjBOVKXcwE1o1Lw2zn3JBs3JaqyRtbEYLWZHYsMFjHiWuhC8oOuA5lCDCGoV61OK8x2Eiqqsr0j14wnPoELAwtd7YpS5YMATRUqHyaRc5zTepRSqo0XE01ejctTI4uxmvSYXt3pzFle+/Xzse2gbcok0hlau4NGLtW96KSqdBHbfcRCNbhXFNQuIpG3OlvIpqhEjcdzw7fvwqX/6NB67cQcyqYxOWzKcpCXVaGB+gQGti207d2F85SrVf2mmyOKoW/+fG3ChPCc9KA1exE1czqfEGoUk6OQ44/LHZb3veMT+AGC5Jj4yyQgajjd5UgUtAotyBDRPJrUc9Xwc0EYJHefP5AXhWOZ5FZZmt4GRtf2YOXEAyRqrQ9P/5qnL0pmBk319BlnOVpMwoqEHBV1rMTYaETTjIV7zwU14/O79qE5EkBo+iVr4InKFJOI06kqYYTlBrGs+9FN0C8sQ61mJwqp1KPYPihE4s7CAVq2CwSzw1Q+8DJn2CbTCONLxAMTAqVbC9hL9mdJZYggkpjBL4MFH87Ikgp8Ux2Xr2YgAx8MOfrZ4FN/83idVGPuWrRCuIDBt5GaI+vQiSqV+qSgsTM2ifGIOE3uOIqg1ETZa6Fa6CMj6cYbYUozgmzrDQyqusiJhsPzAoaeQ7EQxcf77VLtIwJORKBrBi9EKbp99Aa1YAtd88WtY/6rz8MD/7jRjKKKCBDlEljAgnqcAbzYfsCIaTwApVBhVkX+fmplCxGlmsd5imsxTPpVPo8h2Q3YQSal4nNa49yWA09vSInIOBamkqWtI3lSiZcY+4ukraRtOHXWMQM7711PgUD/5uMaE8WN9POW46TUiF1JQ3ZwHJCpXr5tmcYNlwYLb+AHm52dl07nxNWMI52dRjOQxtGI5EMthze9txGwZOHj/CTTDGlLLphGmKCzAUTe7H1y4P/nuw/joVz+BR37wHLLprMTuuIj5fjK5rlYxOTktOfO+npIR+cW+Ms1iZg9ybjxlNKH767+I5PpTV9pU5CzTKlTgH21gqExBNUdrvSnrYEYSjeh05vvwuTVqRH1NsZGDHiLfcPrKPVcOlXgvKNl0KA03l0cFOtbL7TY2vmIcL255Gj3JgvkIxRMS4FP/v9NRz93PQiel1mElEnu99VYMYT7Apr98Be65YReCZgyxZXPYvvMxDA33Yu2atejr71cZdPzkDP74Qz9CmCshXhxFduUqlPoHUG1UsTA7j8FYG9/4wIVIR2fQiUYws9jGkRNtPPfCIew6SKFCUugIUBpDgt2JFf0xrFpWwoYzhxH8b2FlGOuEeDxawS/a0+jEUvj7D1yNs84Y1QcR/Y8JO2+6G5aWiTQb4lT/Y9Rr2Ywsv2RMz0b7QhURDq9X6xqs539bE1Uszs5hbnIarVoXlU4d1z21RQPhBza8G3EaLsWJ3AV6/ZOJDn4+sxfzAbDp7R/BVe+7Gvf8cDuChlERefrZ3GzDjMbI8W22NIvJjXSUw/Ipeseamj0jMvu4JBdwfnZuYUFXTV7uyjUrUSxkEDZ52kQEtFGrin1SBhyCNVJb0KQGbTVa9j3q/AaBshPV2JmMo4+aMZgZejnfYKZ/i/NLUbkupcmOGv5kJ8kLlptdDnu06UxaPRiYFUVNG54tphSqlZp0hDmFM1s7ij+59jIs7JpC34oxBPE81r75fBw7UcPhRybRDpoorJpBM2Kc5obkYUkLTeOOG7fiw1/5OH53024BbMWegtQReR1MVXnSHzh4CIOlQQwMDGj2laCeKW+a9BAXt3yg6EecMraVBTcT5OM94ee0oGHEDKua+Lma+gt7zWqjuNaM/68X92Pq6Gei6w3bmMr2XOeDypVEavi+Xk6HAUW1sPrJZhxebi3g1VdehD1PbhZYyFQ5kTCROZUmEjKI6bkxW/MsQQFFiRwGzhjA+is34K4bdiEVTWLDVSW02mZETtYdA8Tc3Dweefx5fOE/70c30YPk4Cr0rlqHbD6DykIVuWgb33jfBszMTeF719+NPQu9aq12wizaLEVpGs5eD0k/ThPbm7tFKHbAdPq7uWXhb4MKHuLoFf1fIgE2jPfh/33kLeJZsk9IXS8lJBQN4/51Y2Q8+ZQGM/+P2ryrTXU4epYgU1pTcrFTQZFN96a0rchSIkXs9X/xWcQjOew+511IEYlNxkV2JwVsPt7FLdN7MB22sOrS1+Gd//Jp3PPD5xFWYyIPqL4Vq6QriF8mXS7FJLrMyMnWglQWnFUj02VOBFFqhbS+voE+jA70C43W4IAAD6tXKA2zxBJzJ6k3h2ZU5wJhb5btDqZ+THH9VI8GviWMZ20I9ZmdGsPC/KLSSvYbGeGloOioLkojvRgd0XOaPXMYvV4XGGfpvpFeOBNbq1ZQayziirechcb+eYyuWCVdzHV/eD4OHC3jhfuOotibRXr5CTSCOSG4YbuCarmG3r5+/OJHz+GDX/4YnvrJbqSTGfV8+/t7tQhZA56cncKhFw6jVOzVxpV3UoIgVsbKAVd+SPliadzRgpa8kJxgAfWrubl438yDmcGTQw8mSqBa2pVs2szOo9dcDttLhtu+zcTPLyqg0mMius490p2cDBjKxpzDngJMB1iszGGhMY+RoRCxWhcl9q2jduJ6mx1mEjIoo6+U27wMVJVGC2tfsQ6j563GPT/ei77eHoxdyL40Mw5qaidVcbc7EXz2S9/Bnb+bRJAZQmpsLfpXr5a4QHl6Du96wzjuuv1BHCxn0Y2aQAFT4EjUAoyoyQogRiVW1yEeQ8vZzqj99vO3vCn89+eewo7j80rReBrl48D/fu1TeohEUHliGY2R1WsEMTaDCc5EEppEKRX7kMwWjAXDiEqLCykXmJWJ0haCD+VF1Si84fVmFfFOB+e94VrEC33Y8ooPYHCyKlS7oxqpjXoigt/MvIiDYRmRvlH8zU3fxaN37kdnhhs3q7qT18wNzEXGB+4XjG/60+OGpywXDq+BYmDsPVebNSxbtgzFTEapsbxz2GoQsOK4yi6VVapKPqAUEu305P2gYiSV+WUKzjS909aG5EnFfpxqJKVwfsvMAAAgAElEQVTKrI8M9eSC6usr6d+46dRycEPTTN0ZeIiHCGGNxnTikTcrEQMnN0N63uz0jPF/K2VUqwvoWxdivNCLlWPr0GjGsOHai7H3wBwOPjqJUl8BtdwOpPIEQIDjR19AMplFqbcPv7hxBz78T5/Alpt3S962r6+oUUWO2c3Oz2F6fgZ9mX7kZE+yqDqcGQ1TN1E8eZKRZeXacX4+l6k4B+D5JZKFPIGdSbmb9eZn5Hog44nsNAZ31k/MMigqV6FwvVJjk9S1DWwAoszSvIWN3OxscwuHSNsJr00t72DLykh4oAZ1uTaH3qE4Tp7YjfHSiNJ/b5rOZ8uSRbJBZLWlqVNNSZsUFisVXPS2lyNa6MFjtx9E32ABwxvYozdRP1qqRoOkyspL3/ghLGIUieIo0ivWo3/VcnSbLRw7dAzh3CS6kSwiKQZz1sSWLfjxQ3M7sC9t0qXx19O+9+SN/xA+u/sgvvQfN1qNyRQ4AvzL59+PsZF+pAsFFOJ59GRzZq4cJOTnU919GIdvfRCpiRpirQCtiOkwsb4sNQIxbyS33WijFQvQoWp9xB6wTheO/kWjWP21jyJ5yfk4/NX/Ree/7kSE/jsBeZ6U34/hifljeCKYwUK1jU/98LtYrBWw73FaH9KuMo4ux8SoPEH5DzfMwM3Hv1MqlL0dyqUeP35cWkp8XYqDnH/ReZg/OYtChu0Mi+pSqHT1r2aTVSdZFjE3M6eNwpPGo5r8fjLJ09xmWEn898ytdov9R6NecjOSyUWQSX1OCagTOeSMqtV2xTz9hLpakETfuUm0gBIJnezeHlM9c0m+kjwxoxp0anYSzdgMXnXRWiwfWodqLcC5116MFw7NYebZBhKpCCZaD6MRziLoUG2pKetIBtX7f3kIH/rKJ7D5+q1IJTMYGh5AEJBAwpS4hrnZOfQVS0of5QoQYzCxe5FOmqQvN2ahmNMCkwome+y8p3QUiMdxgvO32gQcmrd/Y4uJwZZf1WrD8AgOs0fNq1g9cGk2n6I18Lmq3ylmElvipmjilTL9/LU5Kphel1h97FKwd85yo96U6+B8eRapUh25bheD2Z6l8sXPpMtrKZV0puP2XNkfvuKDV2L7jhkc3VHFslVFFFfPL302ri/yJCqtNl53zXUI08uRLC1HenwdSsOD6MxXsHPLVh0SsVQKMRcUlBI7PTYBul7uibO87A67coT1uqE51FW+6R/Dcq2Nj3/x69i06Qq87hWvxJrly5GqVTBz12/R2XscwZEpxJpdpCi3QhSWi0+9XIs0GrbvGOLpawJC2CJekwni9GHZ/mAkdjsXrW4bfVdegIF/+yxm7n8alQ98E22ieNTNZV4Ti+JAYx6/qh9CtQO89Qt/g/WbXosHfkiyAN+fpxJnNbnIynr4WuBy3DOJU/XhOmactFgpi0zx2t+7HJP7J5Gk8zd5xHSrkw2Iobka5eNwPRFOESVSSCVSJiymuo0zoQlDJWWBZLeTI4/8HUb/VDxp876UanGtEm8JyZ+VxpLukVH95mZmxDUmsslTtJAvGFgjw+cKkjJutv6lpYddCdNxU8zMTmO+OoU3v/4s9OeXoRWmsOGtl2D7zuNoHiZzDJio349uZEFpNgXIZ6Ym0Vfsx7anQ3zkKx/DIz96HoVsAcViFvk8gbEK9u55EaPLxjTN4wVEeL3SOdYEmPlIibXGvr3bbAqCTO2oXhE3v+AKaZMLiwqyslrRYL4NgdBPyRuGcXKKtaz6x+Q+M/X1/V63WW3w3U5gm5F2rbTTZIWZcUpUPWrcaG56Pj9+n6c7sYaZxTm0g2M4a3Q5MtGERu24ljzST2tSormsm0mznCrP4M2f+n384odb0F8cw9gZeXSyRzA5OYnJySnN15JnX2kA//i9R4H0CFL9K5EfPwO53iKObtuBxfl5pDJZxPjaMbo7OuNylRqm3qHzVlguZQad5KvLArXOeAo/f/t/hfmFNo7evwOTjzyDnmpHOsasW+Pqldqu91/EakwEnQLddnr6qQU+XG1cZy/CyMeWiixCNNnvcngLGvLabfVlcdbm76M9V8exqz5F2yGdtCzW20GI2XYdty7sxWzYwblvvApv+ZtP4/4f7bGBfuk/2QynGTTb4uHDZGvIs3EYwVmbd+MhNr35Amx9bCtKyX6zX6Qwmh6ODczzpDaFhLZR5UQggNo+PDG4qZge2khigGTKPVi1vgL1K0ny4O9wMUpkrWvADVM+LjKBTmxZKTW3jVivlDWr2kO+cSajFoiGxqVKccrSlEHSt4p4ijOVnjx5Agu1Gfz+G85BX2EE7SCNDW+5BFuePojudBKpeAwTzQfR7syZ92+jiXa9hhNHT2B+cgU+9o8fxb0/eAY9uQIy2Tj6+3oxMzuFWpmqjD3i+VqWxNPALCK1gLgpnCkVsw1D7g3x5896XjI/L0sE/js3r8Tb2PtlnSy/J1L6rBzj4mdgYGqr9hDnp52ihaW/RkYwn1pj6p1Od9XoJkkuRK3dz3gxRBJYTIaojmarjonpaVTbR9Gfi2Mk14NcIS91EqWstGXp7dW1skzgfHRQiuHyt70Kt3zndxgeGcNseyd+fuf1uPbaa5BMGn2SG/fhJ3bhB3fsR5AdRrJvBXI8cfuK2PrAQ0hn8qIFxxm4nfSP8AExv8wzyXVWrWRz3AdN5y0N1AQIHlp1WZgkYOEGdXkTk2SdRLqId4EW2xrgrKZXdDTNV40guRpQObgWIAegqV/rHP9MCnhJZ0onhtNf9qNK0WQC4w//B7rFAg5d/GEEtRYiBKjULgpQ6TRx59w+7A9rSA8N47M3/w8e+vkBdMuExTrIpvPaELIldBuDCLMhyTz1SGvsoN6u4aLXbMTBgweR7GTRqlcx0DfgVAbsQXHD+tqYf+fD4BfbD+w/q+6MUxzNUE2zrjSyvEYB6ffSqIs5RcoaU0WemN5xQMCDQ1RFPCM6TUmcRgP5bGZpookbeHzlSszNz6NDcoK4z+bB68GgmdkZG/RutzEzexLHThzDa16xEr25AQSJPM7+o4vw9O8OojObRC4dwzR+R9MPMdPKtQoa1TIWZhZw9IUiPvqlj+K+7z+JTCqHwaEeCabv3LsDq8fWIJUxQQKhuKSvpsxFnkGRQUci4uTyOkM4s/uwnrfpGlvQl8xrta6NwI0oUy4OprSYXvJpm9IF00ZmQCwzCGRqXWqEzwKcHywxhpJRHHkP/DXye2rPxR05hKi8K884LskMi1KxxEOIjs9WJ1DvnsBLhlcoaKaiCdXjXNK5QlG6VBymCNoRrL3yLORXDOPuG59D/8AIUkMHUGnPqvPAykrOjc06/vP6B/HYvgCR/DIkB1eiZ+U4svE4tj3xGHLFfs1gRwisatzTmQIwXXakFTk9SkbJdL90ODrZGpvkiyB4bOSCkLmzmQrZEc1tlzDW4lIU5QtJ7cJtUJv4M5sRRUSZe7kBYPVs7YubnI10bmhX3ToFgq7QaS7ske99FomLN+C5V38C2dmKgCARyAhUBQEemj+A59pzIof87a034unHJtE8mUWM9Q0nPNwQv1BhN963JGcTUrWxgqF1vQou8WYcsUQMhVxRtZTUPdyDZxTnBuHn5GmXSZPGZ20HnsBcOPwfr5kbyMQHyCWmf2qIYq6gHrMWdYcSLaS3LeqGciaYwUS9RYeAsg/LB2MuCHZ3fCosAbFuF7lMdqm9UXdzmyZqXlcdTDS2Vq9gfn4ar9y0GrlkEalsEev/6ELcf9cOYD6K5csHMRt5TlRJ8bbpbM/yodXBw/dO4+Of+wgevWkr0tmsfIlypTw2P/woXnLWOTZQTkIGTzFxj01xUKqMGiC36yZQaIi6Dbir1SNPZDt5xc12JwzLCdbTzBjUI03EBdBQmpWL0p/U8qJyLR1OMhmvm5vEXlM4iAsMzIJ4TRL386m8a2fa9BjUGzUKp1F8mTpPLUwjPdBBs3wCq3IjKknYseDPkPvNjIKOgCQcXfiXl+PI4TpeeGoSgyPDSI3slN4VT3c+V5VkzTr+4Tu/xY5JttPHkBhZjaHxlTiwbZumzRKZvKi2HDf0paWBbJY58rqYbfK+MEX3AVL9ZMe00+bVxnUnqMwTnAh1zGECPpIpHQmApEvd/MZUX46ImtIka6X4o15725v8OtaPT1/VdHepTPHj16D3L6/Gts9/F4W7n0eXyvOsYUTyCrG9MY2HascxG9bw0W99DdnhM7HjgSmZaVGs267B6hx+eN+096lvmKhj1dljqJ0gV5XSownzi2kwdbWRRQYWTaqIZ20ax5qPlCg4QRHbSOpZaqInKU4t68eeYo/olLJecWimVQx2Shjrpu5SLlNL5KkwMNinf7f3si//Hj7VXJxbRG9vr4CoQr6oIGR1HeVW6vqsrKXn5iawfl0By0dWIJZM49xrL8evbtmCYtCL/sEcFuO7KBJqI4bMJIjyV6t4+qkG/vBPr8azv96rdlCuJ4XesSzKxznwbm00qmbw3iiu63rtWZMRZpkJkXOr9atUzHQlk2rVGlH0viUQTlM6uieGMHswi5mMSpKWnaDKdCRiYJuXmAC/L0UMJ2jnUWX9V2xdu9c61V0KTZEEn0pzuoeKJJo4Yg8dXTHDphYn0QgP4yVDa5FLc+M6JJktwgQ7FnU0unW86TN/godu24OgkcHAaAnl+GOg7JJlXJZddFpVvO+6X6OaGEaydwXSy9aif2wUzz26Gf39A4ilMzppSSM1BQ4DvtgO4p89ocjfJ9IiPdXWmGGGnAdPLXu5Nq5OR9cz0kZw43Kn6lc7Rf3MrmDqUwerEFWfFnkyOVNE9TCdnIyG6ZneiN1k9R7TreKmjcj/5ycROVHBsT/4AkJasLuJGb7FyXYVt1b2Y7pbwUVv/j38+Ze+hF9/5xmErUByI0yrPEe1WOxR6snWij5kpIWL3nQODj5xDFE6kDurTJlTq/fLn+NpYO0ev1i5wRURXUnAFJjvIzUIjgemMzqdqVRhgZ8zk9YaUW2mE9k+nxHajVRB8gY3Ir9IuvCBj3PK3gyNi8UrU87NzGsUkWljJpMTpdOfSLZgu1goL2B6agIjQ1Gcf94GsZxecu2luPWm32Esvxz5YgTl+A50A+uVtrvUvapJA2pudhg9A8OYeHoGgwMDiOW7mJo9ieH8iGpQa8cwZbU2CVNWzchKLN1ojRokQFSsLvV/GVzabXMSiNiEFH+ezCWjjSY1tOExDwZHsqT4M5TvUYeAmAB72q5V5x3rBcy5AOrTaB0QmtKyUkQIshsEIW1QCDixBtrKMP0mv5oYAi06W00szM1gsvEiBrIJrBkYk2WNTjzO7VIzLR7H0IYhnP36C/Gr729Fqbcf/aM0VntCdS1benJdTGYwNXkC7/z8LxHmRhHvW47U8DgGR0ew9+ktKJJVxdOWjgsJTiNZhsD70GyTi2ClGfeSZwNKtsdbazqXS2WBW0Zfru3nj2058vEGOt1jc9WzNFoTREsypwR1bMSItYw0hAnXMy93spsEUsRNdv0ouRfoxvP/XQ+Q85lDJYze9w2kEgXsuewjoNUwwS+pOyBEA13cuLALk62qdJW/evdtuOfGPYg1yAv2UyVRpV48OUVamFtEtVvDm655FZ7Z/DyyyQwSbLS7E5k3SQU/f96JbJvyhbsXztBMCh1CJCmYVkY2m1MN6GsPDVArG7EbzM0t7eC2qX7wgVYWFxS1uWFtEZtIGiO737iq37xxmrtGKlTy/fj6DAILi1Wl3BxlPAWQUctpUdTHZHoeF23YgG4kjvPfuQn3/HwHBhJ9SOYC1DI7EEQoisfAydqwpfo5VTgXEweraB/rCkAZ3zCKY7snZNZlz6qjU4drgggwA5ykZyjy5nji0jB2QxzS+2Lv2g0fcMSEr8O61Zip1ttmj8bqO9akBgoKdCJgSe4320cJ07TW4LjqbFNT4cv4UT/7Hadppjcw6SANqstnmA4JnB5qOjM3Xrcx1BjcqTDZqDYwsXAUtfpRnLtmDfIpuiPwVEyimMuJQHTRuzYhjKVx1w1bsWzlOIL8EYTJSUQidr3iTXfaqHUDvOPTP0OQG0V0YBWKo+OIxUPMHJlAtm9AnRKbCIuKjimchLRWlWI2fMLRWj9wov3oWGgCsPT5Q9u4OgUdxO6lXsTY0H0I0abDPJFibl9fx0qmxrjBegAauHYCc6KuWWSkNaSLDEsnNL+/1CDniVssYPj2L6PS3499V30GqUqVk6+ajOjwwXY7uG1+L17sVNCMRPD3v7wJB7eHWDjYRk0Cb4YOU+jLZESZZDfwmj96FZ5/8lnkUgVNuzC4MLDwRlMwTSi0Nok9SC4e2o1ysRoZg4CKtSxIOuDgtcUt6znqlHdTLp7mp15mtQYuWHF9azWUeou6LvNqtTaG94IxQTbz1zVAoiPbDn5fPWNJqhiyXK/ZCKM15SOYm5s1KZhqBXPzM0gXFnHROeeh1uri5X/1Wtxx/e+wvGc50sUoKqltQMC+qaWq/Awc6B5ddwmeu/8wEtU8xjcOi0dbjPcYi8xbmDoqIe8zUXXSGvllFi0R3SNeL+WKfHvLVD5Dsxh13GbrRds9NwsWnqyUJDWgy6fdIrQwhXTaX+rLcrTSrRsCWkJYnTqkP5F4Xww45FqgTWdCyhFiWAmLYW+ZiLQJA+rnKB7XbGChXMbxyd1Yt6KEUjov76BcOidKJLOnTR+8Ant3nMSR58soUGu57wDaUng0NVQBYN0Odh+exRf+7QEE+VVIja5DaflqzE8fRqvaRLK3T9x5dll4/WQJ+iBH4pP65Kdlrr7T4Q9WtsqUHfP/nhq6QN5BYn84Lx+lYFKlt5tHaqLsIW0f6xdtusMI/qK2ufpORTSTNd93cv64Ek/jQ1JUMSKXAAYytXqyCN5xBXIf/DPsfc9XUdx2GKGrMcmkYozZPHsAT3RnpSzwse/+C7qFVdj36DxadfJjCSjZbCW/WLtcfNV52LF1J0ppRx7QWCEDvfWa2QKyFMsQZY+amqAYh7TrOiWLhaJtNvn/2KnK00AGWg0j2osUQMnXuBFBuCEqi1W1pPjgyfbhIjVE0NXMsjqpqHfL7wlkIpHekTG42LgZ/ICBwJ66aSHz9/h9gl8kQ1TrLczNTyGZncJF55yPVL6Is992Ee67/jkMl4aRzHTRzO9Bs0WXObsGRvf52VksO3MTnr3jKMbPXIG+oTwWDswikcqphSTwx1ExfW+T/GTW1MwseLKxx8375a1rFNYc51jZBck61YrWjW1cG7D3X6o36zZIUOrrXQpexAHIIdYGVWpLsoXJmfrSTkir62Dw2fN+SczeqbcYW40kDL+5DCBV8NagekcbmVRcDrdPTB7DzPx2XHDG2eZkkM4hmc0iSAa4/L2vxYO3bUdnIY7ScB/i/XvQCo07zo3rg/h/3nAXHtnZRrJnLaJDKzGy9gzs2vI4Sn0DiBd7FdxYz6ssEOEkpj5zwDlhmejBJta4R5bISjbUwnvpeRLBs6MXS3PK+wL5h8WXMHBF4PFSrcdvmK6ytoHzZ/HppRG0pUFMdUd56FqqpBNWEx2urcSGrUuXooko4meMYeDGr+DQz+9D4ut3oJUIbIiBvOVOB3vrM7i9ekA3+8Lfex2u/tsv4tH/3S+QhuR/EgsicdMzHjt7EEi2ML+/hnQuiUTEGFGGk9tMsdExzUTZQ+/sH9oYmRHjGQykc+TYTdrwrs3AB6bo6NJkntr8nAQ7uJDJhBK7hxGeSn6uByn5W6dgz3tNEoI3txapg7alAmH48MwHlq9LCmCrzkDH8bgWFhgcSPbnMECljoXyLMLISVx27gYUV4xi3ZvPxYPXb0OpNIBkpoV6ajc6odHzOBjBz0qlzNVnvxI//taD+PQ/vxeP/fQpFLI9qv3ls+PS/6UA59M0qydO8YOd+L0tNmOK8TPa6Wajn7z3XKD2/Lk2DMziZzMlDVsjptNt5RWvT1iHq/kM1OrqdbSAtTh58jeEa7B0s3LNnrMnZ3AjLAGObhSQPyHMgddIZYw2Qb46dh17DGsGSljZN4I412U8jdKaEi6+9hX45fe3Ih6hYF0PUNqNbruu4Rpz0ON67uJjf38zjpSTiBVWITG6BqvOWItdW55BaXgUAZlj5D+TlEIEmZvVMdKoeWYgccRQf5YFEac9zcNL/043DGJGAYKtIy8/JRbnTkneoBhrU4cE+5NCD1CkDIuYlmqae7g2tJN1JaTO2VprfViPkzef56wHVlg42AO1Af1EXwH9d/8rYtUu9r/hsyJ3sNdFyUve3JNhHbfM7kaVs4p9efzDnXfgwR/uQyZOXWVyUFvSpx1Y04uB0T6UJ+jDQqmUMvpKTP0c2OSmLeQzG7MmPReMQCWJiiVMnFojfM7KwguZuRPaVB1MTpWDF9x81BAyj1x7KP4UlxCBQ1k96YLXKxYPJYGc5QZrMVIifbrnF52eBetxPtBGS71QlgIsU7jJJyYmQLdDMoGmZvfglReci8L4CFZdcQ6e/PmLSNIwLdtGK/8iELAt09CDF4BDe8vsejzyqx141yf+EIc2T6gVR0BJ7BwnfSt0XsMbVOPIngZOmVay6XrZXK5lJ1zEhj1QRJ1fKgeEbVjqyr1FUIe/w03ja2Kesja/a6kjnw0BJVtHlk57tVCmzEKl5QYRA0XTddqTwdRsCzzk/WdQNVzFVFGMJmm5BK9loWxgGjf/8YXDSKcmsKa4BslsHKl4GmsvW491l2/EL777FDLZHEbGc6im9iDomqyqyeoyECziff/vFiyiB/He1YgNr5SiSKNcQaanF4l8QTRfL+fLtNnPWBN38Iw9May5lxzeYofOqUCnTb997NLQI1hEkj2rxxMqfCrp20I+yWFEYP/Nn2AOebBI1zUtYf2buzn8M8EQf9RbAmyRkUyeZUNDKP73p9A5ay12XPIh9FIbi0U8a0m2Gbot3HJyO04kO2iGdVx35x3Y8tAMwlmDzaS4H1vExks3YOaFGW0ioqZ8h9mZOZHmrTfm1SttzMu3I5jSSjZGd8gWmAm5mXyNMgbWbY5AwpuptFgqDVTEJ7BlWQi/eLIYD5kLlUHBojK9l7hYRNhfLKNUooyrnTys93p6Tuk6GzvLakL+TmWBKbLZiPhajekjpT752oeOPIerLtuIgTNXYPDiM/H4z3Yimy0gmW6gUzygul896oap53O079jJDI7snsc7Png1jj1xEulE2gUfA4P4VXWeQAwUlm055wtHDmDQ4joxYNBOTKs7Wb9aNqa6XrO1liG1HEXW+MWnnChIwOCz86eu3/Q8xetSyLDX8/8u7W6Bgk0paSylx9y8TlGS18UAGYtSY8oZRPOaXI3M+tK7O87MzePw7G9x9tBq9PYwkMbwpvf+HubbIZ781SH0DBWR7VtELXEMQViXtKwtGTLaGnj3Z3+GTqIfmcEzkBpbjemTxyTQx42bLPTYmJ6mfeLamL43K4MMch1cGaOSSlrShgdImCAwfWUNmm4feXl4qgi2qGSwtJvGcI1fqyu4QSxD0Wnj+r4Wu2yEzVpJdkrwxrHuM3DAjntLdwzU8GNUZGkN5IqIXv1ypD77V3juqk9gYLYhoriiI1sp3TYemD+AbcECupEQH/vRf6CDFTi0mT24kKIPeOklG/Di9gNIMd0KIwpCSkXCrto+kuVUe6PtLCdYn51Sm2AarDE0pb8eLLJUyNfmekpMs2ocjK8jX+BgudrmOn0NYQzQdhGfC4r3lAuaG5lUQ6tPTdJUJ4joeSbnygejf6OKQpVStTZULgvGtg3b8/e5IaSEz5Oi3cRiuY6F1hQuPWcIoy9Zhb7z1+PBm55BqYeDIh20Mnul9MCNR++g2mIFYTSFp5+aR7cM/NVn340dv9wlIkgu16P+NEE5kd4J7DEIOuKCyY8aCczKB/PbVe1GkobQ0oQGJnhSW2sLyOcKCmJ+Tla0x2x2qe+qk9hZ3XCteBMyOw1t8ovvytdMJ1Ogq55mmsnQ4sL3eINM2hg0TJOYJ7G3pzz9JNe6dVkin5ECcbWGQyc4mzyPlcOj4pxf/fE/wjNPHcXUoSb6B/oRG3oRYZScddbTxuASyFWp4z1fvBVBuojU0FmIJtNoR0IkMr3I9BQRTWfVnvHlmW1BZnYxE6B3Na31cO3z0J/JU3gpV2RYTATB7uWX+oPP0juS8qWImHNop+kpaac7cEWuB/Jk9U71tnT5u+rziQHiCnZaUbqJGp+WKgR4UEi1TQulbB4Lg1mM3fFvOPqVH6N962bz/KHyA8fx2i1sb81gc3NC0z1v/9cvYtXZr8JTP9uNdG8O6zesxuG9R3RTmIYnY0nN2JpfkW0QpkJyqKcJssbkLKAs8V4dWd1HdC4kXic3I3/HpFMa0olmmqcb7ni7ipCyhHSDCm5I3BQdrNerqB9ACLWsP93pLlTcUdx4GlEgTf1TaguTsU7pVf5OpS7wRWkfn4mUIpjutTA5PY9KdwEbz85j/CVrUdpwBn57yzbRGAv9ATrZF0z+1WlwVRfLCCNpPPrQBAYjWfzF378HT962HYl2QmqDYtPBTMD0rH0dq7TwNGacJqtaUr3wih0e+VTG0ek4i1XTRPZZhA+ACvSOJWSKkdbz5QnDTMfzc8mqUkakn3X2ma6OVr+eo6ZsIaq9ZKi9rlsaxca29wFTAcBlVabfXHNGajT/aqNaKWP/0d/h7BXLtH7e+sV34J5btiMV6UWxlEe3j8bW1F2O65mS+cZW4ez0At77d79AkMoimh1BrVHD0Mq1CHL9SHL6i1hL0vAWyxhs4yqbFe/aqJ3iO2jzdtGVbI2RMyRpIWvbLoLdY5cuORn4Rrnl7ZYGKyWkgqH3u3WbTm+oOsZACD4AzTA6cXR/QT5NUprqWiEmoO5qHd5URaEIYqU8Vt77bcw8sBUL190g7VsnbSTPmqPtMn5T2Y9y0MAbP/8hXHTlH+PuG7biyqs2Yd+Oo4iFEGXN4Hb2vCgVyjYCwR5OACUNBVwTb3QAACAASURBVBZTxdIbayNxkTjK2WnUQxMbM7IIPyNBEYmOU2vKjZx5fWhFezkeGEBC4gnvp05HTcLUMDg46OZ5rffosQJmAn7OV/e7YsLs2iDRmJ2ynHBp2YCBmDSRuGprkvZJAaSlRbnTwDkX5TA2MorSmWvwwM1bMTI0hHiuhjB3wG1cowmWFxYQRpJ46MHjOCM1inM2rcUZl16EF+7ag3KVxmj0ETIFCGPu0GjMaXA5Wqef3OF9phm2v07dM4chMHiaLA3rSjs9fGlgizO0ckjgyylfKqt5rT/MZ8ef4wZRf5ZC7sQiWM5wnJJ9Y4KhyugMe/FglzGv7NDxPV8/oWROF6HOH95v/l0Cdd0AR6cOIhudwdr1q3HFe9+Au36yE+lEHoWBJBKDvJfMTo3h5dtRB4+dxMe/fCei6TTiCTouVDEyfi6ifSMIqJsdT0i3mffJNqsRaLS33OGydDg60wD1fV1m1glNxlbFyu6xy2Wz6dnvYgG5WGARsKPepi0kk8Rc2pRehoQbXBMc5tInbWZPtnDRWUgjZTzZ4nBK9fwzazOeIkTQSvkChh7/Dqo7j2L2A9+0XJ7TKIyW7Q5muw3cVjuAxW4LL33HlXjt296HwexyPP6bXcgQhEmZUJdno4gho+a81Q6iw7m6kbWrXvi0TIJPXOkfb5T7XZIguEDYtuFDVt+NKQvTadce0qLUInR1BFt6ra5TyDCghikh081Oq24kFeatdFuv17UI1cAX5c9SS2YHZIEpqGh6hsCSSZuK/OECDBdQo9bA/OIC5soLuOLtG5GLhYiWhvDQT7diZNkoIqmT6KYOgw9eny/oyn40CJJ45rlpjAcrkUkmcOk1mxBms3jx1xOoo4pItItEGENIdQZZUHYQ7TozNUdL1MZjuuwGMvQZ2i2d1Nqg/kQ5je2kZ+ACuQKRo/rZgeG7ECxvjEHlBc2ZLtsYnAn4i4rqxAmWxvHcbDXXH19bBA43G670O8ZAaJJA3PAyg2sYgYanJw8RBt7JqWk8u+VuXPO+N+NlV7wcD/3sRbHC+saSqESft1ljR6Tgg2SgOnhsGp/8+p2IxTOI0Y4iFkHvygsR7+1Hh7PeZJLRtJxZmKWd+nzClVygs31oJ7F2JX/PeVOxzcl1J/R+z/JNp/IehxT7COVTItZporsJ6fPo8almsaKc4wsL0nZv6us3f4PVMA/ow5IU/Ywb2G5uG41uB8v7B1H4zT+hOVPD8WuvWxq3s/QOmGvV8IvafsxHWlh79cV4+0f/HlsfPILeZC+iEfbHDAkXgun6tdLn9Wn5Eo/YWhbyQfVyK6fxcDWvyeEAmkUXC0Zsd+LmYgZpUsoCgp/g8Owp3h+ioNXFiphRsiBh+8MRDKhW71Nj3ikuLO5BSqVaimj1Ne+3MaYog2qRWSqJAjSkD+vaSkTTG3rwi9VFnPfmcWRyUcxMtbHv8RMoDZQQpI6jGewz+F5JGXv0BDwCHDpYRW9lVMBNN9HBS990HgrLVmD3nftQmaUaYwJBzJU/zLAoYObKAx+whNTyfy7NzWSy+oy8h3SC8Pffja1YUD+dyHPa9JEvT5ip0AicbTCF09N+3nAS27Qee+Az47NgENSn5HpUIHTDIW6V83eNd22ZlhFvDPlWQHTWNvze0SOHMHxOGhe87gI8eOMOFHvyyA9XUYnss9aNzMpPHWS79h3DF75zP0BdKOIRuRzSw+chmu9FLEcNK27cuJzo6VniuQMKVk7myPxxA6XiKpe6xlPQHtAZbZs02Ltik1JlS1+WNrr+7ml9HjRQu8RB9aYaYVQvnzb7B8oTwvpN1nc6PV3236N8DE9Gr1xB1Hi4p4TBn34JtVQKU396HQLnym01UxQLrTpuLb+AmWQHF7/3arzkgj9A7UhWxHBq/LKSsVSsi2w2s+Rw5pFkf6O4WQmc8Ob4z6h0x/VVGY2LPTxhnU6wd2Vwo2QUaGMqafPHlkZazQTnWdRFf4lD8fYeZOH4E4DyJYywBvQYuYDXayoQnSWKHj+Hpm3o+sBUVSvXUmV+JZKkQrpB8m6AVDaDcrWMNVeNIozWcHxXGQefPYGh0UGEycPoRg6Ic8yNG+XIZtxE7SrTDVSOlBCPZZCkbUw2i9zqJM561UaUJ5vYvfkFBLWkVBl4DU2q7bsMw0zHHNWz01TdLz8mV9fq+p1mlB9/VOotewNPBNE2toXp5I7swCBK7Vp47nek6OgIPD4dt/64pY+MSQQM1cryPyuk36RX/X23zLGzJAdE8I3BVm1Luhh4NhuDcHYCG1+zEfddvwOFQgaF5VMod4/rkjWwIA65qaLs2HUU1/33g269A6WBMcQH1iOe70OHBtmprH6Hp2087daAH+tzhgOWevvDkWm8gZW6fxF/KAUIdoxcIuaUb9N4YMZQ5FPyofqg3KRuQkhC4K5G8RtXN9ydCL6INgc964fyQ/ovgjq8UaoJw1Ath95SCX3f/gSCdatw6PWfQqJtg/F6qEGA2UYZdy7sx/FUA+/73jcwfzyHZKtHahFcxAQZ1Bvk7zj4W5HX1ee8Po/kMoAwHVUEdEZT3pKT12u1sVHiuDgZufV9iZbbtBDracmKhAQ+TDyOBHUDUMzvxdIxN2rlepCkDfL7cQq7OxE73gu2pHif/KSJ+qcUQFetHrd5VV13c0kAT2qN7GV3A9TbC3jZn23Ai3v2oXqiiYkd82KlxQv7EUanjLhAxDcWaEiC6d7ciSlM76Xsar/xp1NZoy4mA/Ss6sP4xmUaQ6vXotj71CFUjs8h3o4DHZ6yvCd8RubiTqoFRQAJDPr6mOORzA70HGCnndYDw6ysVt2mk8gawSwG3axlE8qcLEngNYl+q6EGYytJh15kC1fDKkMhU6umZ677tZRJOdE5x5MXJuH48nwdM9kOsFit6NSWiigNrocyGDozhvv/bxcGh5ch0ks3yZrxn0m66YZuVrqNJ57Zj2/c9Fs0W1QETSJJadaBM5EoDSOeTCGayiKgeXgyBRYtTIE9wYbrm2uB18z+tIIz1w4F4pzwvxqSrssS7FnOGveUIJXfuKf/ly/CByFUWObXRqZYSkmcRrD6jS414c3kw6JQuPp6px/nLsbyPZQSqY61xTn89Q8iuPRlOPSGTyPXcmOCtO9otzCPJu6c34/Fnjiuu/NWbL5jL9JBj5QCeSOVUrgeIk2lWYP495WcqNNdVr2rVMren5uQ+lS+Ac5/07ifs+10B4K1Kpwxt5HuKXQW00A235ug1RKoFNhp7TeiT8WkHsJ6qlrR0IOXOl0qRVyNaKdGIIEzWb6I9GLfU3bkUkeiokRUCfxU81Vc/ofnY+fWgyjPVjC9awGZQgrJ3n0IIxxMMPUInrj5Ql4LfG5qAhM7ExjsWa9NyAkXm0VmfzSObjxALBVBcVUay8Z7kRjoRTpGzKOL6gJQmamgXWmhVWmjQqvQch1RyuxSmYQ92UxS/GaVMV0GNNNCZl0rE2s6CHAZkxK5pPllLTC/vvg81CEQJ4A1vu+XG+XWgoIBTHxG9P7VkL7zHGJ/l7PAqqdVG1Nvm1NLTlCO+obuvdXB4KQPSxwy/XozOOOSHvzmxi1YPj6Cbv556VJbu8okYw0TCbHrxZO47tu/QbPTFc85nutBduBshNmSAKsY0WZiAWSmxVNyP/AYAWEufg5+ziWlGAES1t9VOeJKFB1Ep29cf8r6k3aJLOFOTZNYNZ4rbxiNlJiqqLZxTCtLfE7l3F7027+mpQJ2CsoYiZQzUgMYvQCs+fjbkH7/n+C3V30UK8qGVMvXp93GRFjFXdVDaPQk8LXN92Pzz3ehlB50DB1rm0jIu1wG9YJ8veOjrrSgXL1gLQMzxubm42fSxpbVg33JOtJ5lRrybKm/r1dVL8m825zn/eSKofM8BZymFJlEro9NYopNv3A4gGbOXMhOtYH9YpeeG2pJdNrECHTiO/oogyhPNqZ3XOy9Pb1YqJWx8ZpzsfPp7Yi0E5hemMf0zjn09GcR79kDRMwzSUG03VJmwqBVWZzG/JE2wuoKFHIEw0iJTKAVcMwDSvOppdWlFZVLtSutefSvGEJxKIV8Xx7pfBbRHO9fwnSOSRqIJBSYEMRRW2hgenIetekayuWGetxBlfeS12IBlKNs3FynCRwqoPN/3IBMmy2F5J38/7P6bE0ZCGUDDKauweOWfV6eYr525ikrySKHJ9izshaNmXzYc+e9oa1KkIxi7aYSbvv+Zqw9p4ROcr+456daVoZL8HV27T+Ov/v2r9FodVHK9yCWzCPRuxpBth8R6pOls4hQNlifk9pqrsxkXe2YZsoKXWnFZ0X7Hz+UQIM67jdNtu1adlloub8tSH9TGA2NIma9MN0uQdTWC1SN4WoypsAk59uiMzqg0jn1Ak+dEl4ZQYigkzXh7zTCNuokm7ebGLzwbIze+GXsuu56pO/5HbKIo4Y2Yh3gueYUfls/jp1hFTc8cj8mJ7uoH+CiJwOqjXzBxL2Y8vLh+S99BqeeR+6sCOzJhNQdlEW0O0IUJZXqanuri63u0kkrzV87qWXYRITcyXiyhcAHL860U4VU0POMKC48ybSaayBTdD4UTkWRgC+dJFfHGVhCAIs6TbWlsUiJqUmPyaReI0EcKVJOM3GErS6CVUmc+fIVeOLmbSiN92KhXsb+LQcxPDIK5J7EYnlOWsFMfPK5rDYJwaN6dR7tSgUTe+LoyQ0hESfRnzO7fPYkgiRtskbsMT5jprRc9xyuoMMhrVhsjI/3Rsg50WvNvtaRHo6iry+P4dF+JEdz3McSGuc2iVLHmeJGHa6TuPrU88cWcfIwjb5NkysRMIvhZ66ArhEm4UJDL6bCMcQ6PHVN75ubnjRVM++y9cr/cdZXgoZKnwlW8tQzQUGfkUnFhYGCZQm1lN3maQYNnP+Gs/DzH9yP5WvaaOOkNg/XNv/LLEvYSLWKk9OL+OCXb0Y0bKGY60cYTSJfGkMrKCJSKCHd04c2a13SOpPmwct619x0A/XOI27dKlsjRTgw+1hPA1VZ6lFlY07ZLK1P7yzyGnOJNYvnzmo40X2JrNF2ekhNytMw728q6nok9RTwZULPnm3jidR8DTrz8QM02EboyWHNfd9GcLyCfW/5HNJBTJukFQnxeOUYtrSn8UR3AX/x0Q/gvR/7azx77wtIVFKYq82ikKd9hkVcooJ8L30212wn15csGm5Y3ghGVd83830/RTmv8+NaHYymBCwYjNQPTtKGkekigTDrQYvwH7OUlgHPExf483QmYG47MTGpxc9eMOs4WXW6WtvkbjquF26iawoiAv8MOCTvV7hAIq4WXZXDC+0Welf1Y9Ur+vHsXS8g1kgikgWG1w7hvv97BP3DGSy0NqO3VNQzpCwLhc15zby28sIcuvUqKrNNLB7LIZPqRyRISXybJ6icnzhS5wYA+JyqlbptaJU/VMCgxI+lpmq9OcDKwDtiGDzpjW5AlFQTWgku1FCDIaneqFT+ewd60bOsoPtLjCKR5eB+KCPz+myIykwV5dkqZidm0W0Q/DSZ1zgoHMishOyziAzCtZ516pLRRz9gBlujD+oEk3KFUU3ZA1I7jrPCGnInRx4IYyHWvXwEyVwCv7zxYYyuqiAar+nAUvD0znyO8joztYh3f+ZbiKX7rL4mFyKWQ7JnJbrJAuLZAiKZNBLpHCIJU9mQwoWE+LtC4Bk0/PS7AN6E9bo9wKqSgJnToXWvC/2mtDrWC3QZUmrtnVMCzR4GFxTvQAFLv6y/JFKDyDCWzrB48b1TkhL0ZwlVGxeYIA0F6ViTVlmUR9rYcNM/o7VuFfa/5qPItQKxk7qxCO6fexG7oxVsCWtYfebZ+Nev/TsGz16LrffsQWe6g1jKUGJDeS0rsGsw5zfOufaV+k0e1G1mX8uLtkeXP9eK8emw/7zkFfNFOdhuQe5Uz5GR3TjAHCs0CiPfn5tX4Iy8ZiuiKdoQvtExfSrD96BAnI3HiVi6BOiJI622Bnu7bTGomMqSUdWNtHHGprXIroxg29070C1nEUsZCj20oYSHf/Y0cv0ziGWO61kxmPb09iKbzmjRzM7OmIl1bRELs9PolNtYPFFEMtqLbpAAurzOtE5go23SGI6v46RiHFAiJ8S2pbFKIU+b42UdZ+uLt8aGyPVcQDqsDYiE7BU71h6d51lmtMIGFluLKPZmMDw2gFRfCsX+IlL5JHJFyr8YZhHpRNCqAfOTZSzMlrG4WAWn7VqLvG/UvzJ1RD6QWo3WKXQ/NOcLtdt4vXSld2L46VwG0STQP9aH1ecNqwW3/cnDmDo5gdzAIR1ZrMoFIjmwVevfWZ1UG8DXvns7Xji6oEDRDRNID64BkgVE4hlEklnJ10Sp501AjJkWNyuzJ1JGZcPqZsV5rQQAHWnII/PKfk9s+P1Q5G9q87imtk4hl+Kq1nNpkicJeLjeCn3H63UHsf7ON3cMXl9fGrvE+KMaIXQSI0JOUVedSznWWrOF9de8HvnPvxc7r/0ickendaM4QHXf9D4NGdzTnkY0XcQ3PvY1jJ03hjWXnoVaO4bdjxxApBJHrEVU2VQVuJGpjMHTdXhoSKemUn1GOIdYE5klt5arq1JbVBptTCjr9Zlqvnn8iEXlfl8b1IEjmgoSPbKNSr0mLi1V/0I29Li4iJYWcmhUjV/MhyCvXFdfM/DZAo8gQo2neErvX+8wXSaS3EKWCov0xmnX0bd2GGsuLCFsdfD4T/c4+46I5GKDWBK5lUls/uUWjK2bA2LzOvXUVuDMaqVGvwCEHTuhpLjI0qfeQKOyiJ/8cgv+ZNOfIuykEYTkc9sAQUvSvIZxcNNVax41tyF1lgE8pSnnw40u2mHcZkltOsurXri5Zke24L3RhtCpbkP6BNx860snE0dFHQrMcoRrqFybRyIXYmT1AMbWjaBvpBfJBIfFI8JiVK86HTLZhEgVzEAv9r0F+vAanK+xDioYxbbdaOD5hw8gbMZkU3L05GGkSy+awFMkoplkG4K3TIIBlfz4Q4eO4Hs334VnDtQZwsUviCRLyJQG0QwyOmkTGQ5+5MWkYk+XG5Y6VAK5JMrIAKmIgxgzFr4SueKntUeDF9ddGeYyabUdZGTlFiWPa388nw4w+UFsq+GMZaTC34EB4ipTv8lNZ3he8hIBwZ2EJlRudXEzbFgPNuyiGQ0RGy7i7Nv+Dfu+/n9I3/GkHlol0sEDs/txMt7Br7uzaIQB/v1jX0dvzxC6yS4GVpew4iXjiGRJK4sDrSjCJk8HXorxO1WzO41nMbJ8K2JphNF1FEXP7qJdZ5pm6gmcYZWSvJArO8m9eBdBllq1jaBMd/MG5mcW6djp2kldDUb3FovKNDrOJoW9Py4Cj4h2OObogBciz/Qt6ka6ohISACr055HuzyKVjyDIdNCttrBt8x5M7KtiqKdfgYenMp9LMhtDelkCd//sAZz9stC0puQcaCVEX28vjh4+gBgBNPka2wLn14kjB/GVb92iAY8zlq3HZedfiuH+lRrcCEO2sKz25yYNWKN1CM5YSs+U2tzzbCZW7cMo2WZ+3paoadK1x4zAYJ2KU3JBasdKrMCsX4mae0cIBVN3UAiLWQI5+WfTV2q362h36+hwTakHamm3viJsxcSRpH1KlHW4PSNtPjG5KDnEv0dRyPShHdBDKI1Sfxbl9hGE8UOmONKwA4G1NF//FJ7BPv4ifnTrA7h/60nbuNEUooksOpEU4mwPpfOIJXNANI0wFkUik9WwPliOsDxJmCg781kebrId4FbzksgOXwr2jb8mZORh9OBp5E9IRk6fTnLj+pTR+LvuPjjqmT74aRxlGfY6Rgk9hITeOoTWvE5PQdsCHtp127QUCIuFmE408erHbkJ11xFMfvBfEWu2cDLWxmOLRzCR6OD29oxO6He96R14xXmvRiKSQSxIKlK2Ig0E8QCZXFILvo0W4im7uUbnNObREmLOWiYamjGx5nEtbbHxPa/9w5TqlEoGvWH4JURaEzG8f2l0YvTR5YJzkx3qJSt51vuKJ+3IzUorHbXN0HzdeaGd5plGlhlXVhP1Kqd/aqhNLWBxsoGTB+YR6SaRjtLhjqbSRYFC2ggdo0SeaNBs+RDa4aJOr76eXm0C2Xa0OavcUrbACO8VGRKpFF7ctR1f/96v5AgnlROWPd0Qf/eZD2J2ahbxsB8B8ohHc4jHUgKXCPYws+CJKlAwZJukJblVugOIEqna0thewh0o5ytDcvOrEndX/GS3Gdg7d/RO8aQjhgxLTldahqwJiXSzlWQIPrEYvk6jabPOtAzxd1aWrG7diePsABdDn03RhFx29li7aKGnj1NfZFIxbW5henEPXagta5CAuRt6d84XGnSwxjJuu+cJ3HTvHgfwkdGXQDeSQDeaQoqbN0GQLiOnSyLNiVxRzz1wptogW44ySdpfUQ3fc237+WhlxIdWXxUKgiZClzAdYZ2gblLDn7AexJH+r++XuBpSJAueRg6V9pFRQIqTqVEqtiTqxdVgabbQSKncGfBSjbYwv3IAZ97wJQzGsnj+jR9HqtXGweos9qKMnYk6HqjNoBW20Zsfwpc/8LfIxPvRbXQQxqzWjCdipmFEBQ2nB9QmQZ99uyXhdvrmGhjEyOz1kj3t0IgWdhLwzzwBTe7HNHB5UhCgoP8rTzI1z9VfNAQwlkgtSalSgzmItJHJxhBJnZJtYaYh4I3AXtuE7DRZFdCexCRRO23LaAxEsTpI0rJqZ5mNZ4qqGZx06obIkPUTi+BE/UEgUlZfUPYligbmEGAC7yYxRBK7mFnsgycS2PnsNnzj+7+wWVG3mXLZND7/6b8wDnWtrs/FINBX6Ee7TiQ2jk4zC3SziEeLrn4n+GVtQipJiG0V5Wlrk00Bec8aZOHUi9W7PKlZtrCmlqE4gdEEHQrpR2TXw3tPwzdNn7khA6G8zpuIa4oTPv5w4X3jdVsZQvle8+ONJ4nSG1bBHrOCClNsAVdRAxejATKFJOa7m4GIlXnqtWbTSv1tHt0sWYzV1ZY964nFDj7wxesRTWTUOgqjaWWBNghFz6AC4pkehPEUYsksujECVQES6SwLGGV3IYOGRNJDeRglSP10bUNlity41uqhKJshhNLuWSS7x3pnVsSbgrpa356f6Taxd7iTlKk0h4xkoO+zfhEiSpZSzKlBOjE5L7XJfq5DqKvxDpqXno2+T1yLwtgwDvzBZ5CaqeBQewEHIzXcWz2KZ2ki1m2qyf937/scVvasAuIpuQcqlWIrIEqxO474uTYWWwhSUDDgbH6e+kskHKSM8K6Nau0MEUm0qU3DyPvWaqjemTl7gomxxY1q6cUD9G/OrZ3pFEESD2bF4m5mmUikhgusD9jsniLmE120wXFj5lg7xtBFD1Aw0MlqlKlVOqkNyZ+hoF09mEYjtUsqItq0Lr3nHDQXkhhITZqLdRFo8H3psMeTv30cP/zZwzrx/cZljfeRv3qLpchNow6yDUIsQwqP0k2i/lIMC3OLiHTSaNS4+eJIJ0tIxqkYGbfgGjJQMEAJ8zeBcmY8HGSQjxNJElaOkAyi1pSzDeH7MtUnF1rMKUer1byqgpzxvokb0ErVNpMJ2BsKTJDKSiRxoCUxy9vRQYp/56ZN2iy0PWumI3XMdx93oJGVh0K83bPjuuHPk7TBzUfLzocefwb/+qPfoRkhVZHrikMaZHExFYsDHOiPctMWkMwVIUVutk5V8yYcvZHkHQY1m7xiNsQ9qq4PD8MD46/TIL2QPjfGxmjDWoZEAd40W6RWH3qlC5EWPHFen8XYUUuULOcd4/Sil5QTtJmdsJw2uU5p46BqwDroIv6ZazD01jdKxXD6+tsxd9N9mOlWcaRTwewlq/D9Bx5U/s9ToTeSw3Xv/yKyhT6kYvbw+H0pChCdcywtcn6lcOhoY6rR2Cek4DVrFvXPDNP1LSwf4bSxGk1kc3kbR+w0zb2BKWCEFhxMobgZSOE0tQKbG7RJmWj8FDPNNqoRMrQAOKSeiCuFVbsmlUaHYmeOyCL+ruOu8nc1OkfyhZwBTAlSp7Bn/rRbqCdeRLxQA8u709li1BLmRXHThkw7WUe5z2ttszbu+tVvcMf9z4mkwV3Az7tixSjeee0b1DZJxpm+2eepafiE7x+XM4Iye55gDHydDmamZ6V8yB47NyxlhlpNysxkEA2LCNjUDSOIhkl02taPVXbTNuEBS51toF4sK2czyu9z2oqGb5wgUtargX/7GTHf3IwvFwNPcUmcUpeM7TeXjrOeFHU3ABKphDZHPJ0QOMn1zM9WDXejHhxUIObr83kR+SXzjVRbOtAvOvBTfOlYBB/7xGcx3RlGNdqLWCSp+6PWFdefDAWIHrP2TiCMJHTopLJ5taH47/9fW+8BZmlVZf3vG+vWrRw6QneTBQYVHRUJOuo3I8YZFUEx66goKDkjsYkCDTRIFgUEkSAqCGIYdRQwIIIISu5cXTndujl8z2/tc273//985YPdXXXr3vc97zk7rL322gwDS+nnlIsSKhGx3yMOoeh3ZPcPtGKfojFqIjTtxgeusFlT04LguRL57dqO4kYP5AAvtTg8TghIDTPSBymoi3ARYPTIDtJBwVpSyK81bPlvr7KRF161aqtmuf4he+HTJ1u5UbMtzYrlv/RWu+0nj9jf141Zg4OTSNs+O+1jX3r/J6yne9AbYJgTaoifR9DCrwFrjaaRqHGaTMCDzDjAJmTZrZnUG4MH5uDJqMlwRbV5B1WElAcBPH5WLkFIcLYXG0rN99JXinxpVz9wiw56CuPGmTDq9y370Gcvv7iaJOyhaFjZeC71YlZUGaUlfrPSSvVhdFgyW7J654uW6wYN9snyQmlbXG9d18uhFN0XD5xwMYHYW3vHrT+wJ558SYYvigS8ad/X2Pvfe4B6jCnfSRAAY5HBA3pzgZd4PNJSxMakwqJL2mgNYCwJ0S7q/rlu0H4R9MFWkgmbnJgUXpFJ9zGhzVL1y/y6HwAAIABJREFUTrN6v9YE701JLZPuslKZweCUtEgZyGNTojDiacm7iQoU/QlHcEWXUqmiFjkw4FoNdpLz7om4cE3ZbEJiABrfyhC9dCepprVyz1ijWVSFgByYlBCvifH0PNsrEDJ8taaNT8zYcSeebOmOfivl97FmGvZTlzSaLQmZBcOPYcrK8xLxNJkhjfgx15/rsFy+X/zubDavWdHqFmVSvUYf+H+JDasObkUScyXMXIkhL6CV2FDBI0YChbsL/3ISfkr0NuUxyoucNyqGh6Q6PTSGu+FRG8OeXAmwrWEsQY2mpT+wvy0657P2l7cdaZkdBm3VDafZ4x/5mnWUKjbS0bTmx/axzlyPffP6222qxJhtl4x5/35vs4P23d/6csstkcxLJZ7jK/qbRN0CgyvkuKJ9qvGBHMebsrlf5TzhcHGt3AeHFMMFwUI5OShqmO7HnNoIuPB9Ne8HNQiXbM1aMsiPKD8C/NAEc0Jy583y+xpwFQAsKSHEBmtNf4jAjfNjVW/X2ru6RI5wLJG0SmvW8ssnrZ4oW7az03JJJ+YrjggjWAmXNWmC6QREDu2pp8z6Kdn13/q2vfTqhDY4HVx8ffKwD9juuy4R8KYG+UxabKRCaOogQvN72jbHKUZTrF+sKDh32HnpGuoVBPoQiuf9eN8yRAmVV7ps6+iYLVm0g6YRZixv1WpDOTSH1yxjzToN9DQ05ARMcV+kN/CfAXZoXRTIKu1jmH6UCEO0E5r6FWJrzErWevsGLJFCsYW8c8ES+VetXJ2wzs4eJ8dkMzq8rXRWDRuUGDu7GRA+oAFt1VLdjjvhRJuaXWAcgaV6d7VCcrElWlnhR0KXpS4CoEk3G4AUDQ3h8JIDE3FIi5zSXpdl8p3WkevU/bglotRllti86/taUR6k3fcY8gANuQ6eJ+Y7ejSxKyjU5QTgBEE15/N6o7MeHlY9jF5EfS+WUvBwEgoK7CbqWQtLu23lPRfYlnt+YYVLvi9v0H3fBbb1+4/Y1I8esblF3db48GtULx0vVOzKm+9WEg903pdJ2wfecZAI7r3di9TMvFBJ2pLh5daX77bezn4RCogGsGztHAkgJBIHQqnB64aAQR42x3owhwSkNBDUnEIXROB8spzrbkUxNRk9dSo54uvyr2EMpNDnbfNxMWSy3FJGCLNz9L2QB+sgU7pxZJBpBXwWXoxQvNwat6W7t0RwTyMrCkDHbCQJAzipXymPAMG6NWsVhbEwmmRLBTA27ao119q6DUi9Wps/fvYZx1omSU6cFmod66tKRwJSLCMdpFecNBLeNxArFH1BtkFzStMJ3BjyOjWuBG0yRWgQIrX2TStXSpYipUh3WXdvh02MT1mxVFDDAqEu6U5P92Kq0daRzlujlrZmnTIVOXbKki244DCmcqEkaNZqJK1Uqemw8nwi4T+XT6nubNkZa6TGLJllVnLShocHbW521lMjvDaeMzDdxMuGmVUq2ab1I3be6gvlQYnkrrxmrX3jkttsrJjzHBcvrlZqB7UQKEDhJEFKB91L3VLqnpfHTeIMldfCwmKfIn2TEVKf2LDy3Tq4nps55ByZIO4cnT0lVYmga8ufPDCmA0TPKog+kCviQ3PAJgh3ydM5isyXI4d1a0EYqDatvHjYdvjZ+bbwlxdt9PMXWa1W8gHXHz/ABj/+YXvmE0dbaZ9lVn3rjtaRzgps+P0fn7Cf/vbvEkFLJ1J26H8ebDsOdlulVrHRqSn7ya+fCMqLQqiUO+XSHfaFD/67dXUusVymV/cFcum9sRwkV6NQqCpUzw2Qiv/UJhM+psS5o4B+7oFwTmxqDoka3mWQ3EJXar6JfVZRUSQIb3DwvAljIFG2MFA7lekUKOb5l/NiNa6TcIuylXJgKBQVG5sesVvvW2uXrDlLlEHCdcA3RRNBJsbfO+TNQmKhpTI/CO/mHl9pS6Nql152nY1PzIu8oKjIzL76pcNt0ZI+AS3VMmNMaPwvWk9Pv0Jf1irqZeu9Ei40KNlWoopAOIH0QH4psC/pAgc+LdGnUYisH0j0GPt8vlOMNxmFMP2PAxJbM2nw6EOZpMUYWGRo8cQcCed7K3SnqQMZWqYaVOr20AO/s6mpiu20bDdbvnilZTJdajKYmhux10JvzBeF1itqKpdCAwkH0eVk4bk3NMKlYV3qKOMMEIWZrV59qW0am1KE9G/veJt94pOHCYD7yhm3WLHZa0lEBQC1WhlLZ7g+b5CnPV4TDpizVKPu7g39hEmIxXFWUmlem2yPn01sXHVwK7a/uXV2TxDDYB3S0J4WgSQXqHY1x1gmwkT7wXfBK6G57nv0ED3E9AXhSwghsXu5bvbZf7eBr33YRn/6Oyt84zuWalat1KhaK52x6V0HbOdrzrKnDznW0oe90cqD3knhIFHTrrzxThtfQFKlZZ2plh313x+3cmneRka22s8f+7vVSGCouQUADkNy9Gc+ZP0D/SpBqLUrge4zfOOSUNcowQqIA7qraXoJDh3IZNpaVY/5+X42xxBqJ65kssiXcvhZP8JuR4Ep6WgtABViCCxEPkjdaJVcA8tbCYPUjvS4XNpFggPNhm3ZvMme/efzVmnVbLbARPWmGFYnnXGMLVm21IaGBnWdAvqkEBEGlyn4cjCwUa/I4HCASWXaoEerYasvuMLGJuYUVcgAJxK25pJvmCUrVipWrFIuquXP1RvrXquVfKQ/b0UW8V5DtSK+fyy7qQElGEepVgRsRfcYSl/CAEI0wH2o9Bb0uXU4SUPCVADQZxEUQq0YOVRE40HUWXOEzhFWoL570YVX2eZN04YIP4CVcI1Wy978pjfaRw55V1t0XDKv9arQZxBjUiL0onxNMCTegJJN422rNjszZxdfdoPqtRiQq9eusc7OjD366ON2y3e+bTa4r5XTSy2R7LSmDqU3FERD53xlBUHWEM8Aznc4i4jo06sF15oDzjVv3uk9LZgtCmEDDUBaSm01gqDIGObCbl/XBVSIobSTWNw7RQ6o8rSgNuBaVds2CWB183W72ZKLv2z1xXlbf8r11nr4cWuiHs7JBNxKJm2yp2W73LPGfn/lWut+80orUzMLnkSDnusNu3jtbVZRIGe21y7L7D/etp+V5mbs4f/9q03ME9pGzVqTNTv9a5+1VtMbDBQ5AAjkctJIjhxnvBQHUOUX1au91KB8jUhB+TxgCG16jvyyMVmfSLrHKLCJhJsjiwrpQU7ca9gCIeH/8vfQOkk47fvVDzC9uL5RWlarLNjzL75sv/7V0wq5sEllapbNlh1x5BH2uje8wRotn0b3///yFkG8d0rv44d32yRB1iGZaNk3zrrYpmeckM+9otB54XnHqwcVcKi/t8d7mBvetxrr/qrZB5X+uCElBk/Yx9wjPLV4uH5YolfTBIJQEhPfuwpiT4Tns4UiCBijvIijRDIHNWzX8Mqonu31bmicTsaQvG8I4zHMZ5xxkVUqAFYJNcNw+EGM/+tD77bXv34n6+vp13NCk8taSOs6FRUGkz6bZ0GRJtT3wQF434VCyZ57caM9/ue/2gc/+J/2tgPeaplswi688Ju2dWSzdaQ6rdq1yuazK6ya7vNGnGDoVM1JYLS9RIaFVfOKhOadtAPSzIZRmEz0tGW397dU2lGZxEO6qObHxtIhbHioHBdN7p3NEaQ6faO41i7lH9BILaAGbLUsn0haIVUXwpy1rI0N523n606x1I6DNvO3F+wfXzrfBsoJ6yDcTDlaizebt7LNZLO26q4z7YU//84qNc93/OFnFK7NzEzYP9aN2b0P/14PIJNs2pGfOcxymbr99ann7HdPQ1NzwEglK0valz9zqK1aOqAGb5DcwcEh3Tebzw9MnLVLmQrShiPpURfa4xsvX4kwobEbnrtiqWmfYwOCYMuC8qlhc8awLzZpyHNrTKWLmwnND03aMUWJ10bP6sYN6+znD/9eD1Oc2kbLyvWavf9D/2n/9q53tsPKWBVo52J054SculGc87qr5uY4SAcVMZlu2WmnXGAzHNwUYFXN9nnta+zzn/1ooDnWhAADRnHQi0VvZ9REwoWFNuIdUXBeV6b3NsizAA5JjzuE5tG4xDq5YyUOXqkc1nA5XJEnQsqFkwF0WrR4kXdKpTM2NzdrOcpDon0CInUoraEWy570mnenAKTTTrkwpC2OHWBkcQDHn3iEDQzkBGIymRGVDQxbjJTm52a0p1XHD/wDFxwEXUcDu2StTIdSld1228tq9YqcwAknnGLJRsu6u1E3SdlcJWkL2QFrDPyLNRLeiy0pJbfVIqwANMpwJiCw8HlEE+TB7ky0h0Zf85/AAG04P6KlEagSmpbyZBzrIxJGQD2jNZP8SMo3Pkajo9qyUqppKRQsyM2olQ50Wd+h/8c6Pv52a+Sy1nh+nf35xDXWu2HaOgiRMklJ1TToP1T9sGXVZMPG/nWJ1d/zWsnAuEay1495oFwrG4b2tkd++yd74rn1eigrhnvs0P/8d2tWq/ade/9HCvCx3xVA4F0HvtH23nUHW7FyRXuwFpZfPbsingfeqiyrh/o+jdDXKW5MdVKJk+tKDIpZAlPLJ+wBvhASbScuH9IQFp+NHME68jDE5eSJ4yC1MHlBZQc1MSRt8+aN9qN7HxaAwUEEZClWy/aGN7/JPvOFz7cxBO2D0Jboid82AKgyP2OVYqFN4eW6kbKZm5+y1eeusVIZTB5/nrKDDnqzvffgg5yjWy5Zd75L9++dVC0bGxsTe4swlwNIIwYGNWppd1ALRe0j2+GkmJD/ekNBRgeK94pfhPBKDXgeQWhBIX/CVEJiMBpjVYRIB9aXk/Pxslmxqij7eT856VTDyRnNhgQWzjvnCgdnE16S8464uq0+/1SrVGbV0IEoHNMPCaHFvZc6p0eXfG7/4IDNzxeUg09Nzcgrwo5Dfobcvb9vUPf76KOP2YMPPiIwFRwFeqeUK5Mm9tTXTz3Nnnl+zH7+u2etmuxRyZP7zFLfFo+acBlHiJF2aqpKhOyxrXt8UG42InyxHuetWWF2DhBjyMFizushoqOf8soa7NywCt4tlbfGULelX7eTdb/3QOveb2+rZxNWL8zbyJ+ets1X32d9r45Zg+6UVMsytTDs2qOENkd6pitplSMOtHKiYnXxNgHQOLx+XRC6YymHDpNLrvq2lZuEl2Zf/eInLNtYsO/e80uroiKhPl0ecMpWLem1zx7+YXV0KB8MaLKoiiGP8dw9KCuQW4mM79ROHz/p+Q7ibz7Eyr0qG9jZWA68ONjgTQmx3hdTCT+4/uVGMciqBE8QsYE445Ue2OnpMbvz9nusWfPaYZl5Qo2aLVu1wo478QTPo8OwMJDbOJ+Jkgj1ZeiD9QpNEOTyPlyK1/f09Nr4xIgf3FLTWkmogg372Mc+bG964x5+YDS20g/cyMiILVmyqL1+3HdsPyMHjjREMmuRIljj4DW3XwcOffTWREDkjJHKiPeNzkFSMmGWkFjeQWxO5TFAPRUBhNK01TKIIiCqCJgSaSNvxxx9ZqjJO0OKEg+G+vQzjrUEWEeSCAK1EPSrnRG3bcZuRc+X+49RhI82wYgmbL4wKwB02bKVVpgv2SWXfFPItvSypOjZtIVGRVHCRz7yETvgwP2UBnEQy7Wm/fXFMXv06Y326pY5a7Xy8rKNZMPBMHXree1ZSP6WPT6g+6UpQPUkTS5rqd0IF69NhwIFAARehTfBK6FG0D9opXzScsO9lt53b0vvu7P1vWE3a0JHROkBAGTrlI3+5Vl74eYf2cCWCUvXmpbBgoiUHtkgnuxHaZLYjTT5nl1t+rWDCr9J2Fl8wrLYi6m+23TW5/dIkydpN996p+2//wG2bLjPuvId9sivfmMvbZxTWx4sp0SyaR2plJ175jHKVfEO1PrQMJYqY8aBoFhjxkPIy6sjxkGVTJDWRLMpJ3kWz1lbLZeEAQkFuo/AHd7AvbUr9XMgvfHCQzXPD32wlw4j9cFORxwhDhB68/1KdcFSiQ77/f8+Zk8/8fcAfDWsSG0y32GXXHZpmDcTR4iGubNBwRLomzzXieh1q5aKYqoRTUDIGBndYFeuudWKiLgHIbavHvkZ6+/zaQYeaTCipNump6Y0FnN8fMyFC8JYFU+pXF1C9yvlCTfGiA9EA+b32Gld+bzNzsy6sEGpqCYPfhaNIx5GgntCrr27yc27A1QKH5NoeJUsq95hNrP/DmGlS/Y2rb9/wDZvHbXV513Vlqd1XnvWVq1Ybp/93OHaG5AcYrmLkBnecFWySt5LrnUI/bdxSh+lrpjrM2iMa5iZXrDrvnWzJZNZGUX6zXlNVbX3nJ122slq+O/tdVGFqenxtjh6odK0YqVp9/3qeXt+S9GmFlrWQjkDZU6xv+qWGNnjgy1CMMJJVIYWmg1LQ+1LmJV6MpZfscRSb9jd8rvvaLmVSyw52G/Jzow1QOUysEV8kjj/y82WbeOTz9qGX/zWEk9vsNx0yTLFqjXSZpk6OXQ9dAGR7AddWno7s3SZBMoknpuSSm/Wip95k82kK9JdwjPyoFm8uQLMGTaBWXffgA6Kt5Wh0le0cpWQrttKxYL9+S9/sz8/s6mtbkC4lkulbPU5xznNkFJFBklOZzl10zNbZtSHz3SN+SchICEX5Q/Kz4R3YgIVGG7sWldcKCwf6S2HDhYMDRzwKFmjRosgi+LSrp6zcCgoNThzykN195z00GZF0MhSOrOUbR0Zsx/cfo8sOb9XrbZsslywK69eK/pjDOXFtQ3IcIUh0uWSIgcpKyh3Z/zGgkLCeq1iU9NjdsXl31EDg2eZSTv55CMtnXZ1TAAfNQJIZM37ZQuFBa3bkkWLdI08lwLicFLmN+Xh8sahCYBDENVBkEzlIGfDNEKEyksLBT1jhrSNEoYDOIn5tU0TTOURFDxqNevt65PHJiVD4havqq7aIDKPfI5SmUbTXl6/3m6+8S4dZmq3KgV2dNiH/+sDtudeu8i4w8FWGsOYmS5C4cmQLjniLYMRokz2zczsjOfBoU2UfURU9sjDv7G/Pvl3HUxNWgy6VGTNr33d3nbwe95l9TrGpsN2WL7cJiemvZEeIK9WtGwiq8aCucKs1ROdNjLWtJ//+Vl7ZbRu89Zjicm7H2hl+rots+OwZXbocxK0OvcJo5qWZLQDOlOlqhUnZqw4PmGFZ1+16rqtNr9ui1Vf2GT5essyADpYA3GAE+qrTVVduUI8ZCB1SbHAYnIKV8yXQQHdUnqiPtOTsspn32YLncyLQYXR66hsHhXwo8wLaHjKNWdzHZ3KK5B5RWVidOuIVYolW795iz34iydDkd+nHCQaLfvmxWfoUPK7CwvzwSPkdIidoOJhr8TQOVzBa3Ko0VjicIjHvb3MrIZGeV0T1DSyn7hXCbABPqElHco11DhjmByBKZHVU7mgtJgXM4rrUSN6kvpx1qbGp+zG625p85OrlYZNFgt23U3Xa21iGCe5sEACATBsVEGSg/QJoTlaX+UFKxYWlMNNz4zZVVfe5m12ut+UnXHmcd4QENacziLWgC8iFbwjBg0pHQ4sX52dNEl4VEHLJlEN3pZD4ioZfvDcM7fkwbhvgUWZtA42/8ZYi0KriY7uob1P12ca43HRv8bgOSHfQVS6wHg23jCDyob3mj/x1JN2//2/CGqWPpWQ8P70U08ytlK9XtHBJWTnQzNpIqKsTU5NKoUSSxA0GK/ZRe5e9AaRQOGN0xtY/8suuVa8AOZE8QBJigTCZdJ23PFfs3QGz+nenCiCz5EKB6owRHFBuB5RORDnUrloOaLBWkrhf2Ju3dOtRKFszfmyFbaO2PzzG2z2n+utsnGTNcamLQ90XvN2JuW8tGSFso/mnQSqIIOs1QGDtwn0t9gGFSelCUmNyhPqg3RVBcKiTpC1tNnL6ZrdWt9k//3lj1oyBz+1oBwml3cAJDJusGoKM7p7dCDiYGEeNCijxHGaTXv2uX/YAw//2SoisGdU68tlknbc146wFSuWtjVx2QnaJELWyUfTVizhdX0mTSQ16MDCOop6VMGbxFolHgwAAtlOVSbaA5uh3/nnx+kKeE8JxakU41PpIRiwebhXjd4gfWm1rI+pgPB+az6i8/qrr7VEM2nZdE6o6VRx3q656QZvRQylJZL9tnEMqDYHq1YpSeGhiQepl2xiYtx6u/M2OrbVrrry1qDVxBpk7JjjviSkXrV9zQRyCiiHj9p2rL2io8XGXLJkiU1MTbjxDqJt5K2E0vLAGimSF/WP+wYU09CtZErfx3vG0lKt7lMN+Wx6a9nc1Mw70WzSHF6vZPjfnf/b3d3lhieTViSmAW8yFFn74X0/tl//+n8dmMphBLxF89zVJ2ssCXk841kgzfC7maR3xnnpzjW2eXZ9vd02NTWlZ0sEpucnkgwRUNNefHGD3X3Xj+VICO9pKPAGiabtuc9u9vGPHyrwy1NPP08Ab3FWcmSjOcbhyqS+5kgCe5SSeG6PtwsKVfse6ozUEUVXdM8oUCGIyIlYEb6ilKWHZZENtY18gcV2fSHPdfiSWnxoKxOoxWGSQkHT5rIp+21y2h7LVNV1ctzXP23lwoxyP5DCyelpdYSwwdkkbHDQxu31o8i5uCnQTz5306ZNCqXuue9X9uK6rQpRIXV3pBP2mcMPsX/919fJikt8K1Abe7p7tOHkeekU1fDk7YTBlB46M0oWMqhO8Dr/ooxCCcOHNbdVNxDOzuVUQBe3JzBj4uKomSMYxO4er5UK4Q80SgwDh1bheXHB7rj1eza6ecxy2bzyp9ly0a6++QYrl/zBik4phNytOmR4WX7CZO6rUra56Rkb6u+2mekJEU82btxs1157m8+HSpjE3b961OfE12G9o4ER2URytH6v8kKI/pUrAvyQ5CFHdxpnwuhKwqty3RxSIeSphO200yob2bpVLLA4VMw1rb03Soqhkjjy0ZzbaKo+xlPU1bBm8IsLCz5cnIHogHA77rijQl0OELjNjTfcbM8++091FZGeYYzz+R47+9wT5Ol0LyIh4bmzNjc14cZCpT0veymCiXTe0LvuP3fmE3nyfff81Na9ujk0X8AdcGNKmnH8ScdIXkh2MJwnnlds1pCoXWjMiHs7dq1JXIEvDu7fd3l7S1aFsC/U9IDO1U8r+UpnSMnbhhm4PhOU/CUucuhOidKRQdlBnxFqwRqiFUTW+D7vV0iYbUxV7c82axtyLWuB8taqNl8u25v22MkOfPt+uiHCRQgQ3CAT75jAjuedmpy0TsoMCcJaNk2XvFFvLzKkjNPskKLjn578h11z/d0CJeh3xOO+86C32CGH/Jdeo4bqQCBwEAjrTtO3o67Sygo1bl8PBxpUXwxsp8ikicin5sCGecB8hq83qDRtW2HMYmjUj6FtDGtl4cXEIkzyMN1HZjiSzAb+1c9+YX/+wxPSLyY8nq+V7AtfPcL23nufYFSo/XmPq64tWHYRSAANaxWrV2rWrKF1PKcG/C1bR+3SS66VvCpe/i1v2c8Ofu/bVbNeWCjKiGZTaZuemRGxnnv0JndXT6SWyWu6uvOKFiIqTq6D2J4a+ANnm9fxO/wuh0jN6LxPB7N4UbtwkbyYctAJDnjFmvhasx5+cJU/57tEOxSpRs7AmzHUxighw7RdftkVMk6u1AEWkbRlS3ewI7/+Oe0Xyb2GUidhf7JJia7Te8nTSf3J/YpNTg7c0+1lsXAu8p3dViov2FVrblTLIt6fL5whTm+XXXaxQw77EPRkPQNO1PaOh3uSgQ57UVUGxoeKiaeub/f+mOAnV+wvBQyNDNmuTqlDGw5mRNO0ELh39ROzeg7wYVFSWB+K62yMhtecKImQm/Lgs8m0zTYqVutIWWrVYivsucieWZixB37/uKwPYIFarMIcWcCco796uA4PIbl3eqRs6bJlsv6O/BGqzCssZTMPLxpqgyIgeXScIEX6ysYNdu7qa62JymDSB2qtXLXcTj7xCOtI5iybY+yDK1q4z0zooWB1NOM1rIUsv8Izn1zo9V1XamANfZN5eAXgw0NwZNkR8RgWubfmMHmOGz1tO3pRLdhJJuoECaqP4q4GttfLL71sd91xr6WYUl5vWalet30POtA+efgn2yUUNTyEkp6Xspz9QxkOnrLVncIIQLJ164jNTM/bNWtv8vJW0+wrR33ZBob6LUekEuIJs5r6pNUvqwPheeXM7JyQ20gsiQO4AXySrIU2IdEAtVWXtVUzvlKUvA5ftiNjC0Fz2mv52wZno52t5pagEaWy5XaypdK7Ar+AaqoSl6tYoMpJOMuzuvTSK2xkZNQVP+T10/aW/d5oH/3oh937yXt75KNUp4bCSF4RF3I/7DkcCRRNwtply5bbxo2uQ6W5SY2Kbdo4bnffdb91dOa1z7jGBdDyjk779KcOs/7hPpdI6uiwhdkZvYb1Y9+7MD8sDJ/J7KIPoSQLkh0ObfvgeumD2l0gGQQ5mfbBDQQAWQNCXWlMIS3kaLQCZaRbRHxvWj3RsGZ3hw5poydrXTsu1t+ruy62Yp4e06QtTM9ZpVy323/8U1kVeMOIVZMPiNFUqdgXP3+IDfR2WblGWJyQFacPE4V58kg2zfTMhKw23+/M5W10dLQ9e2bz5k120IFvs5nCjJ1x5hqbmCyo3MB9dHXn7MLVp1pvvkfavpoWD8ocvK3fO0iqN1XH/IwHyn+RqhgPrkJdqX94Ez3kBCeLeHPCtoPrDClZ0TAwTQIFgeIWYiEPP4M4t09m93wsHtz5uQW77JI1AlDUcNBoWe+yxXbGmWfrWtVmp3JJLEU5G00IbzphCzNTVizMyIsNDw9pzX7/u8ftlpvv1OGrNZt27upzLNvhhzaWSBhDRxrQle+yufnZdhrEYY8jVLlGNjyhJZUEvDkGItFsiNwwPT2jZ0Zk5GQJb6cEwALRlv5ZKMl5bTuMlgxhMT+L6UA0hrl8t68nayREPtS5ywBOXgM+66zzbG6WecKu48R6nHTy8bbNwWmqAAAgAElEQVTHbjvb2PiYT2+kbioEuGEtkPhwPaXinMpy3NPs9JRyV6538+bNiuqUE2dS9u2bb7NyyaRdRaQoDKBRs4HBAfvCFz6pzq/ubk+FIndcVYWg8SZCShFcB/qnt4xGFpw0wMKA7sSTK/d35hT/C7pRgme2G5YVaV78EuPsherKEzSsmEtasi9vM4MZm+1MWKMvZ4munKV7UCQEmnc3T7jXSieso5W0JkwUelvmS/abR/9s6zZPhPpgr1WqrrqByv5++/2LHfDmfUUOTwf4HlTW5VOj+FjgkKYResuKuQNwwGKA6BFi1Vslu/CSG+yFFzaKLcRCQB6/5MLTESG0RDpq/3rYFVMBGRKQbMm8OpLpBBXnJgtICdPzZP2V6/ng6HSH82SVF0ZBdhD3KNcjHV5y3RD+BtJ6BCZ8j9Jp40oeYglJRdEbJiDqX/7NK9XBIpwgkTJY2ZddtbZdP465UvTokigNk80b1bL0lCdGt9pAf78Oyy9+8Su7796HZEQofFxw4WobHO63uXkH3Pj9DjWsu+ffOjqqTQuvl3VgPRjclksnbX7ePTAhfnFuzhqAKxna4jyEZeojXkXjV6gpKyUCw/DSGOuIlxUoKgka9lAct+kgl7P5/J6kl0bomWH2jk9713NGUUTPqmDnnH2+Vcre9+yAUtouu/xiGRfRDquw8ZjMkFMoXFVJ0D17MuGcZb4Qkfd+aq+5x9IXf7/xhu9IUL6js1v7gSiO/fXJT33ChgZICXx+kaobNKyEFEZaz6HfV6qkgVYcS4UukO8OUljNn1btTzFGVrWaBJpPqkgvACKMOaynTPKoGbxfZ8LSOw5bZcWAVXqYMNC0Enlp0JnFIuFBgemxQjQnk89I+yfwnRU+ohvVqNvk5JT95IHfWJ2ByTnGUThyCsCUyrTsy/99uAAgWtpU9gHgSbvYF1azo8NHHPKzwWFU+BMmnWg2BS1lTXpgG/bkX5+ya2+8y8OrdEpDmc5ffaZlMjWf7RsOXDLrVEIeOkwlQvToIWUs2sOsIdlT6vASyPZfHiIH30mdMhA2hH6HAeGANF0AY9IiJszzsJqNKHazcno2Laiq52SIrZFSeD9x07598y326qsbVQeVbEAyYZdec3V7M/D4I5LP1cQcmmiJjQzIt3nDK1ZamNdY0J8++HP76UO/0rNHB+rKtWsFVM7Ozckjo1jB78SRK+R3ceNFD0hqUi/7QVe/q5kMqBpCirOiHgqdpuUTAQMqDYp2+Dc9q573aW5wkGfNh1nBUs9QJxGlFUgyPgiN92Y/aDhYGPzm+sxuhAnrp6dn7dxzz3ckmoMIut+RtYsuOl9MOxpNpECCXnMBbe2MJH6IxNi/1JcVNaEXXXO6LV/sryg88be//dN+8chvJHkjrx+ihaHBXvvoYR+wTqIXqZsglMeM3EhqaVl3l3tz4R3pjMJm1fzDJM34HCNnPvHHnd7cwtPy0DPNhC1Y3aqZhFUHOq1/r50ttWzQios6bKZZM+vqsJRKCPhLn/ZO6xGAUnFmTjfCDBUAGG6SBwBXlUXhQuK0MR2erIeCExMT9rv/fcKm50loIIZ3akwI1rhaL9tZZxxv1qhYoeggCP8pf8h3yqry/s4VLdvKVTvpYKmpXZPbQCPr0oJCauTo486S5ebmUfM/7ZTjbcnifpVFWEwsp5DYdNqe/+fztu8b/lVhqELHunNWI7I+PTOt2T+AYpE2mZVkTigBCb111g6GUGUwjXRxcEHzlkLfJz+LpAQeFrVr79bi4MY8mfAOPSQUIFnPhP3pj3+xe+75odg+tIpRq117443tvBlvHRk98br0WVnXqtq8ZbO8R193p8Cq226/yx7/w5P6/XRnxk465RRFMOwN6qHkwXEEJmvERoNGOTMza3vusYfPBgboq1VEzKDEQTPDYL+TZGCW8ewJOVkqjBesN6K7GBoDAsE+Ep4SZtDyORFoEodZHGSK+97dJcE5rpnwVwbXx5FieNl35KCFhaKdfsZZDsIS6WQyttPOq+yYY76mKIz8ER0pDNj4OBEg+6aivcs9VUpFb2EEoKOVr1jUGm4fyn/rmpusXKyLp43KhWZEJZP20UM+YCtXLRWSrxwWOR3uLxBvyHdhyEUBOtdjdsCP/aIDLCDO8ReF0D//xCEtDqmhDtiXs3R3p7WyKUH7XT3dWox0i1EIiGjCrmqoN1HaRaG/dH52ToyoqExIo7dCmHTa8l3dbe+NvjEbnwslb9V8n0TCRrZM2e9+/5RALjGOArm8VK7Y2w58k711v9fpYLF5RLKoVq2/H7JI2nKdPfJaGJHFixZ7eNZqKnf76xN/sl123lldSRzcY084x8pIodJHm8nY+973H/aB9x3c9m4sipBO6o5SE3QtJaGjgafsltZDajYbQnGxtxS0efsDIotMbTvwmmWwwgQ1IdUB3o80Ov1uQPCrNe+KifmNpD3xEhm0f/PWnc/bhvWbhZSqFlqpaDzIFdddGxQPGS7shiSGlfF6+O7gwKA8VKVcsPmZadu4Yb3dccf3VYME61i0dLGdedaZAlbmCgVDXoaNxf3iDWP0gAfmGivhcPmwNUf0ObxEFYipwWQDvOEZahpElDYys6WLh0SiIMWhTMSG17jJYPw9WnMRPkJuIiRI/YpaNMDc95rTTltieLH5yUHZXzxH+mVPPe0M77flNR05e8c7/s0+8MH3e5seTQjzc0oFXC8Mj1uRMdLhpSxYKstg4JW5Z54/pSUiBwz5zTd9zzoynS5HKxS8rNz2S1883OqNsgw468PaCMRUq6x7Zp4vh5k1rtBRFSYVOlaRUmqnUme4hsTdV50gVDnmWq6P7GR6nwgeWDRhrqjC0DBqMlLAiO2xevwZ65E6BNKHNRsaGvJJbqGJXu6e0LzKFPaWHvAjj/zOKlXCVAJF16SqVetCHo86+tPWCrNyya+XLFtm1RrT2wGuvM7a09trvb0Dbs3xbI2GPfDAA/aOtx1oiRY6S027/Kqr7U9/edYyGebpJuwtb36TffmI/3a1ytD8r4I5qJ7a9OLwMsZpOgMGSwuQoCl1msCHd2H+q5MouG4HojwfkuVvxfIPyGWwoGrf2zbdnVBRHTTybhkh4gJhNNoyFMI1tCorgkAuD/GkaeecdV7IP/01qy+71PqHBkNrpQOlMe/2afF1MaW4xl133VVtkYBGk6Njdvmaq2z9xhFFJa/Za0/74hFf8p7QdFoHi+aBXKeP3fBD5uioDkJob4zElMgG0kFGqI/QmQYOt2xG+BtLTGAlDgjVrYqGV5D4ZSN3d3XJ6GYyQe5Xapo+j2lsfNzXDGYZ1Cf1EGMQzdcII0FzQb5bA9fOOWe1vJy8cCppRx51pDrEmF5I9MM1k8viff05IgnQtMIsA+U6bWZmRocMCdresM+Q16GL6re/edQe/+MTCnmlJ8UggEbNPv3pw2zvvXe16WmQeL4f21aJHreN/4yht3L60EEmkC6kEBhOTZlkgDhVi/uuObkVw1qFs6F1T4AMlEAU9rarAUoJPygS8HssUHTnvG5qckoW0KmECzYwNKRifDzQcVwjUphefmlpmNWr6zbbU0+jLuiWqMyhltSF2XEnfjGoaTi6uXjJUt00KoPk1gIzmi3r6xvUweUQR34s+QjhWrVcst/+/jH7zq3f10hHCuWrVq2y8847r93gz/06Z5q65YKsMNQ28qVysabQT8oP9Zo2sTYh4Av86HLRXnrhBVuxYoUsJyGfT1v3QrsAIrE6nSmjNY1lJrxPoiUghTxLXGV5fS/bOLnDSzTpVDYwqqB55u3Ms86xwpzLw/J12nnn2bIdd0Beyz9bAE4YKRkIIXgtrpEQdGCwVyDMb375P/bjHz9gY5N0ppj9x3vebfsfdID1glXMzwvlx7suX77UXn31lYAB4G3CoLVQ22ctZLBoZaPHN5SveM+a6Kt1l5RVe1/Nli6lvFfQurPmZSbC5xgxilF34CmrAV0enemrCXhZsE7V2hvyiqD/aooP9whyK+yDWbSJpD366B/s7nt+qGgBh0LIf+FFF3o6orDa07CFwoznrgCkC3xG1hbmZ6xRcafE/TJOBoWVQamNgOmYXXftjUL2yaupS6tslO2wo4/9iiRtOSORLgu7bHx8XPtGHPcAlnluD+rskR4YgqRZG6RSOT0v31tpS/zoutP0xHWKQ7VOmyBMPI8oq48/SFilVG43F7NIGkhNrYr2JkTWVOf0dii+D9sp6i3zQDSqEgHrvC+oUFRr2dxC1X7y40esWk04Yi3yPCFVy17/hl3tfe87WA9d6KqEV6HI9Vg6l9UNUg4CyYtJPIsDQV2zS8slhV8s1rHHneyT0TNJhTHXXHOdX0NonueAsHj851I7XjZotpLKQ0UwVygPcJBRzy8US01xD/kQy6cWuJCLcX/R+6YgNwSryibyzQkguC3MjkCPb0Lvc63VaMfjetzjduTz4rR+85uX2+io0+94/eeOOMLecsD+Mn7xMPtu3/ZvnmE8uJVq0cZHtqgDa82Va21yqiCvdPSxR1tPX6/kQjl8REwYLs05azo7jY3mU/x8OgCRi9ZfIuRueGK4qrpk3YXLBZIlUzrAgGQ8b9YYY4j353mR/ij6C/OdQKNBnXm9lESCogp1eQ4uho9n7FGiYyUut+vo8f0//In94pe/DtMinGNww403WKm4IGE9ACmuNYoDaO01+QJJ26rVSs5LJoxm5pK8ovp6MTglu/ZbN1pWoXnQA6vV7BOfPFy5LXVfnS9IS7wnTADx1h3gigYpEjA8vHf6J9zmeLAdJA2i6D/81knbBNFbXjNTzlKtiazvVoa6GjWlpC3Mz7fRZiycgw5Nq4fWJiXRKbR0nUYoRJnp9Wj+hG4QaQdlUQsoaaI7N481ee655+yfL4xatZ7UhqEvMiJrR5/wFRXHKahTKlWfpoj+PCSGNBesu7dHh8sHOIdZP5aw/r4+bRYOwKc++XmrI8Kd8qL5TTfdFBbc5wBB/YtKA3h9X1lQR5hAgdlS9fxTOUk6pfyGdYNcHz2OvEoYiAaY52UD6rEgvY4WIs7m5Y5Y4nEv497ZzSgally3jEmt5DlzKmX9fUOSaHnqqafse7ffpWfDfwe881126KcO176OdNNISfWb8UNMGAioRJfQxNiIjW3dYt/97l02O1dUnffiSy9VZ4/wCKaz5/PKAbu62JxJ/RvyC+5ZXOq+PkVnkDMkSBBCZ1B5rrcQFDK4K6UjQbxBjQW0iBKtTU2FpoqEDQ0O2uT4RDst6+/vtSnVT71dDwNOvk00ghGgzZBGh8hdJtyV5yIlq1TtqquusY1btjgwxXiXzk67+OKL5QyY1xv7XKVlVnP6Y2fe97eoljVaKoOkU0itYh5//w9/ZOvXb3ZkO6DW+a6sfemLX7Levm7tEcn9CE12MM0bKraNo+G5eoupH9QIAkr5cTuGYvx54t6rT1So7EOjfAHFvcz5MGtHvJj76pYB3Vt+zmHmAfBhqqSQPwmZTSuUxDrr9UFMjAWkQO+slIoOC2WGnm7mzXpozWu+e+u9VqxQLvIcG5Qaa330cUdaR44aoHsyPodwiNwTj0sNjIkEg4OUn6DN+dgJXouxIc/m67zzLrBn//GKroND/oMf/EDXIoApCJe7JU0qf5a1C6oDHFxnS7EYgSBOe5tANi8NcB9x3WL+F8svbsx8IoTYVCHfUXmMhxoeGmkKX3pg8pQujIekajy4IMmICuB9Vp9LyOcHvX/xMvvG+ef67wcOefTwsV4vDrCZjY2N6v0mx7aIVLB27Y1Wrbm863nnn2/1pkcVsSdWWEgKI0uI1yHWFsZbpUTyQ6YFhFDYm098IBpeyimOHp6LeBGUMMnbMAYYAg4/h1czk8MIEQ938eaO+rqQvKOrGhpGDbhSUV1YDKka2ljz4qjznnGvnHLy6TZD6EnbZSplb/zXN9rhHz9cCPb8grdoclgKc3PtqQmkPzwbPc+sWq30rJUDlwDQEAJs2IUXXaLuNEeJHbR898H/x/bYYw/dWxh0IgfmIvnOVch1ODqtMlgoHUXHyWeKeRV42yoTxUkW4AA/vv40HVwv1nuNy7WCUGrfNjdIag4wi/CaGmhNw3E1CHr7DF2Va5Ipm5mb1aLNzc956EKY1dfbbufiQM3OM8LBgSRR/SgJ1Gr26ONP2LoNE1YLTfuiM5rZ/ge91d75rrcp+S9XFrRZevv6pWkVwwfCiojETk5O2tDQsCiOcDCx+Ljq559/xdZec5OzojJpO/PMM+0t+71V5QG1DYa8kzXx8ZGOMjt44iwf3q9dZhHAFLS6aPRG/IyJ8YwuDeTzapm82FvL0uHgAn6p40gHFAzUmzH0uRTbA9E/Ug3lNYPkKb9TZJJ809Uy2ZTcj9Q3Mx122dVX/X/qqzwvv+4QliXJp3P2wgsvyivNTI/bKy+9YNde+23xfTvyHXbOOeeoIcKHbfuoTJ4/B5c/RdmbR6DAPB1ijnC1IoMtFDuUv8AHCGWjvE3M310s1nNwiBaRaIBnivxdZiupdVIhposbaFIC/HKh0i6orxnFjYbKiKw/xgQnETuv4CMce+wJqihoHEjC7Jijj7HXv/71Mi5TM5MiXajxo8kAbHdUHNyobKIeayKnYtkG+7q0z0g5Nm3YaDffdIt15XtEBfY6f8OOO/5oH5fZpPfcjS+/42lZMHA5Fw2IXnR7YEoOY7upltsaDvyeEw/edLom0vNUeWgcRh5SpeYgFDdBmMvq4WFBxxYtWuzspECtw1I6WuZeyEsk3iBeXPDal8acNCBtw/0sW6HoPGIvMZS0gbjQdes22q9+80erUKZrJKxKY4JCtqyddfbp4tmqnzPwgBl1QdM1G4LWv4hww+jRjfO5INQoBtYrNj251c48a41VkNbs6LB3vvOd9uUvf8XQ5/Vaczg8gWYXrSHXuD3yF/NgSjryyGqccEK7AJVAT8N7VGtlARNqzIfJJaCFHCq0SsqaekikyQZi67hahg+q8rAX/EejOgFkJsfFn8XSX3zJFTY5MacOFkpGV1x7jVNRG4HrGmYUsWEIDZkRBELK88Iw8iypp6+5/Ep91g477GBHHXWUJGzdw2+n0ZzyziYMrufeNevr7bPxsTGV2DD6TlsMwFU6LU/IYRG4Qm0fWVUiGiKikJrJE0lTmbZMP+jkgLCylENnsoqaRke3yijy3FnnOC4Go8rokZg/I2DOvlAE0NVjR3/tWCvXvO2U91t9weq24By1e4wCXABq3KJqUnopLrSbIsQ6C5GKxuWEkPu2m79rr7zySpjc58+PMtOb3vpmr90DPtW3lfboN+ZecSzsUV5DM76GnGsfeVeUkzRcjCDiIE4KImopWuL+605qyVITIlc4wB5+IE7FQxMTRU3AziJxJoeLo8F44cN5KpAG+IBY4lHZgf7SojcnYzUV3nZ1e100gF8R/QVM8k00bb/89eM2OVmU/AudFa47lLCvf/2rQoMXL17i0wPZiEHrSXlXl4NTkZjNdYs5E8oWE+OjlmiV7fgTzrPZYkWh3YqVK+3yy9dYPhgO0Go+j+ti80Rks81cCSFLLF+ogyhI18a/c4oBkCJ3mZqsE8QJieGvIHRmVik6F9WNg3teR/C15GFwtkdBrpTh4SEHpjA5ZoXCjOqkd/3gR/bM35730Y8dWVtz7dWqxQauR2CseY0TA7l5yyZdmyRiBC6lbMvIiJ1z9rm6nje/6c32mc99Wt6Wnmc2itrN1CEWdLe0zgyy8kFvhbl5eV5+Z5aQlAMS5hypw6bsbCOMuLxlC0ZVT7uvNYJlvb39CpkRoQMzYM9QNqJ8hJGP4evGTRt1L+wnNbS0kK/13LFWQ9cpTuZzreKTTjpNooJcE597+RWXK0KQqkqomqhvJmA1Cl0hFgklJyWpKIoU040DVfcG+gvPv7Dd8+zD3lp21tlnW61eUkO/UPXgiSXXm9vGw+bCnJddUelRxqMEv6Gse4vpHPfP+/I92HqS8OXgikwgAGTbgOGFEghdWtaNeqF7gzC+IsD09FjyPW6I8gcfIP1gkcC9JQtJDh2AVktkdulM0UDd06XEH2OANSNfZWP193XZ1ol5+973fmKNZlKhK3U8NvPb/+1Ae+97D1Z+Se6LkvzwomF5D8Lazi7E3wBSumTxBdhElhIGoNaw8bF1du21t9vLG0cEbpEL3XHn92V82FyQDWKtDKOkDp3Q3xqNAmsRv+dKBXHiA43mDsqR15Jrce+cVh/9gZcFkeTjIBP4a7f/UggehMBleDRMzZUXiDrY9KxHvUg7Hn20DXvyL0/Zzx76jU8jTCbsyuuu0WhG16JzBQ82iCis1rLR0RF1WLGpyDG5TzbELbd8x1566WV52z332sNJFqE7is+ltkzTARsIYFEU1nCARfsLJSnm6cxMz6jDSnsmIs0IDII0Q/VUzXSb8kXctF5OyQqrcKTXpWR4koThfM+F45taX4BBPCvOQWmR69/rWlj70dExYzby6aef5dzwTEYp2iWXXqIDzz1KDxt1RdRJAoCqSCPhz1CrGDANX1GR/Oyf//yn3XH7nQFdb4gAc9BBB9p73vs+9TsQusOum5mdFEMs18mUQq84COOobxsMxxwnDBtGZXZuWpEb9yiFytDMT5sga4G4ROK+a7/egg/LFHHGR5JtoVAfmRxYd+QwY60MaJsF5IHHflz1m2qaHdaxYLWq53wc/GLVxc548EPDfSqao+bAgsVNUw6EAKkVZDI2OTlmjzz0R5ukKRwVgjINED4I6tRTT7RMh3t9lpB8EkOhnKNMWO9KGfkcxsQROlngUFeemZqwf/zjH3b7nQ/pCWNxb7zlZlk8MYkq9PXStVIVuX94eJErFtJ+RoknoIYxD8UgicqoRnifL0w/L8DN+vXrbeXKVQrTOejRIkdiS7nITFW/Rr54QP+vr1hHJ4SOh4nWwnq1ZPNTkzY9O21rr7pRJTJSiHPOP88Glixus4TwjKqpJh0sRI2QL+RKSQ8Iy7xs41QPDvj8/KyuDSOxZcsWb1ur1cMECBo9OmxuZla5JPeve04mnSSQg7nkHjWi5uSbEYQkdfGKgHsvohzWGw+4aHhYQgaEuqC4eN9tRtIUzipCCaCh6K40uLfQiMrLGUgFZWbWZqenlbsiLnDp5Vdp/TE2O6xcYcccf4wNiIo532a+8XzVNBIQfcpSNIggqgciiYpHviNnKIqyRtdde63WRg30zLhNJ2z1Bed7ZCVpHs9rOzOpNiLeaFRUfyZlIn/m7BD5lCrwsL3pIIUogbrfaO10FUhPZcNgbdoh773may1kPVAz8J7clEZNxB5QNsLkxIQWQECFKGVu+fk3C47FG59gqpmLuUHL48Hye9mgesfGIQfjcJJPefzuvFVChsmpKbXcMT0PdtE/nltnf3jyRc/VJHHqXucbZ52qh04k4DfX8sZ3NHXzOYXGW0e3Wi4LTxWqGGULF+vmYJYKBdsystmuWPtd1+LNZOzk00+xHVfsqFCPh8XCc10+bNlVPQh7hDzmaS30NrG4+QgV3Qv77BuF6qLRhQl2otlRH/ZZw95p5MoQymuCp/p/HVwPkx34wxGLoMEkvZq3zJWYElev2PnnX2a1io/M/MrXj7J93rBv8A0eDbDRoM2Nbh3VJEM+n4MLM8nbEL0VL/KNyad5VuSQk5MTPi1AFEpU9f3QdeUcDebvHCg8Fp+FJhKbkL3BgSeagxQzsmVE/160aFjPTCgw6RiIrAAwNI45wI6qE45u4+9iULy0xF7kOvEu1H5h3oEjMEYGQy55n9k5Ic3c49jYhN1wI8BbS4DboYcdZu/6D8Ta6GiiH9mbHdgLVDk4/D5NsiXPWpFcqzcTSKY3mRIwdd655wZCBAe+Zbvttbt95jOfFV4SU0D2yuT4mEvXUtJr1dWbrJp81gk/XoYEvHTtZv5kHbmvPM00AsYoU7oaqgz5fdce3apX2YQOJiCVUqnA8vDGZRY9AjAiRouQ4P1Er9ltd3v22We1+IRo/NxHS2QUIgA+8KV8L5HQgnR1d8nqR42dWMfDUqthvcoGX1BR++f/86TNFH0qu4crZq993Z526Mc+JiaJM6a8zolECRuPmySkW7J4sZeCFhyBFpCBNW2YpDAvu+JGWyj5Qn3ui5+3fV73Wh20vqDsEPNNrpP37+sbCF1CPk6D+/OSmDPLsKw8rBhKcai2jXJxkoI2YzikGAQYVarnBn3l+Of2xImItup16FYHWRzJ6lTKNj81pbEjay7/ltISNjVTDd79/ve2ZUw5zaw76wi4SJ2WNQEg8Sl+LlPD57Ou7im8UcA9QkXAIsaRkJpwm3vtyQMgEa35v2OpCnCKr8iv5fDDQIu1Sjaz571QZXkGPsRtYKDfe52Z3IixTXroyL1jGOJzlKEALESSNwBhQvxDnoih3mWnne2Vl1+W89i6dcxuv+MH6osmGrhszRrr6e/RffAsqQGr8yxwChRthV5q+MVk8gulgiKABsL1Xd32x8f/YD+6//5w/z6U+yz1L3fI+C9avNjxFgFoqGEWpN6CAin16VU7rLD5BW/KUDtoEBfUtI06Rtlr7ZhKjKaMYI/PupJ0zU+/fVqLmTBC4zro2ofHm9GAXt+I7iHYTKB6tGjRihfDHq/jegmJw+FcXuaUer21p2dAi6y2LRYGLeHAuGEzqCVLdL6WzRfmlQ9pYnqrYX944in7x/OjVmEqedpJHb293XbBxav13rOzMyK/C2TBK1a8yM2GIQTiMEUDgbVmU8c69Y03f8f+/txLlkx32P4HHmAHH/xu6+vvs54e96gYEl7L7/tA5pLrUwk1RioFQgnSn46eR+oaD2J7RJjr4Z7UtRIQ4TYVUt4UL+JhlXtfD4vcUIX+YCHLXprzdjYyE1oXG1YpFG12YtQe/MmD9qcnn1MueOA73m6f+txnFa65IcFD08XE8KtuMb1UzlmAwMBByYikQgcMz5CwlvQoKkZoh6UAACAASURBVC+SEkH/43rk+UM+SwgevRVejnyT/LEdjaj5o+agWda7feTFa1V58mjlWGO8L0aDOinhdyy38QxUMgztlLCgBKRqaDrcX+ezc5iV1kGlRXJWhq0ksPPvf3/OfvzAz6SAggG54OKLFFarYSD0BUtqKDSTKELo6ZH+tkcTC97ZQ5MDnq9ldv31N0qQn3Sq0qzbrnvsbh865FBbvGiRX7uqIR5xcT/cg6JUzUT26M3vAyVRE/9a1Ev0pQuz7dIqpU8MF3ltR2hukOe984pjxJwCmMp15W1gcFjaQXNsiNlZhTaEJdwIFgO9IW3UgBiSvHMBXJwslTZnXQ/K8ycHCbBmsLG4CBZLeWgexYox65E19noobJxicd7ynTnbsHGTPfAQM4MIq50yxvuffd43dD0YCRYAz0EzOGmvqHVwWRcKMjQAV4AvhOdszrkANjz6+B/tvvsfVqQxvHSRnXbqqaK+8X5sBJUGRM9DVBxpWK83O83PhdnxRHikeGij4oFCaU2x94ZorCehspPMPeRct26dyi4R8nedLydH+rQ/jzAUVYjh4oSKgLuAWklxEw8wsXWL/f3pv9kdd93vSoL/8i92/MknesN7kkhnQSUdWE0YEAyOG2gOoYumYzGGBwd0aPk5fFueLZ8PgwyDhSdRKae9ocu2bNkyeXEOH69nraenprVmPGcOJNEFBkM0UhH3TfuBCfQYWW/hc2mdhbl5pV4idiDVO+PyLjxfZv8op+WAhusA12ChlE8H3jKLRW7KYRgfH7UHH3zYnnn2eWu0UgK9zr/oQoGp0VBCc/Qw3eWLMKZCxRnNku+y6ZlJIcystcA45FcvXRP6fVMqWR59/LG2eNlynR2+aPTwqMCxE0Jw1aMR7gspBevhDqDiUxOC6gc1a0lEaY4VHG+X9eV3wZCkvf3zOy9poWTAg+zuZS4M9bmqjY2O2+v33VcbbOmSZWHkxBIdZh5Q9DRelHdVAw5jLJ+4En/C6kb4hYQHC+IFfTFjas5jjTKm8sLE9QxXatRsfnbGCsVZe/yPz9qLL48GnVk6+ZK2/4FvtcMOO0xIHTKX6EvR4UHIw0bFiMzMTNnwokUKUdTMQFRAaJdyZHWusGBnnEljdcv+5fX72Be+8Dnr7emVdQUQEQIMUt2ZVyTA1D02NS10WOfIueWQIsWC9RaIIhX9jIwGQEcElraFwV5bFaQfDmhUN9jmdd3jKpwObYV6n6DOoVxTSKvXhefmpm39Sy/ZFWvWqmtqaOliu+iSS7xnNXhcnDYGLl63No8+wxs3+OyB3h5dGznm1hFyYZPR5sACsoEroBtNWI3UC903ArDKJeWwXsP3ZnCF0t09WnvYSbGOT2TE+5B78j0+FwPGSBNQaLI+RNWef/55HUZVPIJUjdaX0D6R1IHGEHPgqDDgxeLEB7w5DqBaKdmG9evUPLFhEyyxhO3xmtfYV486UjVxDDPPyidUeHSj/aJ2vZR1hjY79gRccgTvuL+nnnzSHv39Y1p9bB4O7+TTT9VQcVoNcXC0xHqjjosvSISePxs1vQfeevkOy329lf54aZCcXcYyGCcL9EvO0sycI+g4ocTd153WciZMTioKkCLwZIRBLKZD1ynp5bJBPY91hDDX0eVNBrS4gSTyPbwNYWtot+vu69Wh4X1HxyfaKhiUYQiZgMyxfj29PbJWqO17aapm83MTesB33/ubdkkEz8WDP/e8sx1NTPiB4XdYJEI1RlosX7bMNm7aJMALhQi+6MFkqgB/0lj99NPP6KDv+/rX+USDLMp83TY3O6frrahTo0fhEfTHWAYiJ+MACGCq1rVhooavuocqVX2PA+8lrj43dIEhFi09axQNnyPOHh6367ihruu58fajM32TRaQREGdkdL2dc/aFyqcGh4bs4osusmTG5yU5m6elzc51xQYB9cuqVu2gGpxh8AeBlJq106VNRWkHz8i6cj/i0Qq0c7I94anWX3IwKRkCn0CfkaFns4k1FFBrDvusWuW8g4fmj5WrVskQ4+mXLl2qw6Mp8Gzmri5J0PL+XpGAI0AImbGZkJ+yRgpLg+wMnHPC6S2b19uN199ko+Mzlkhl7OD3HGyHfvRQa9B2SQlIE/e2TWpk34lKSQoHSYTcWuW9ps3NzOi6rrvmW5JaUqkrmbQTTjzB+iBTwGnPgrJ7js6e4F5UbQpG2IFCJvwBotV0b6Nbt8pB8Jooy6soJCDnRDviXTcaqm+zfomf3HZhi2Qez4GahLOjGCkYpu9Rv2V8paBqs6VLlkpAm79X6VlVztohDwOXVA3QeLS5eW3KVTvvpA8Tb7fpJQJCy9l5FDOcUCA9KknB+phFrCULB3+22Sjb9+96yCamPETnogFaPvXJTyjsmZqdbOfXbChH/5LqDIphFtgWjfcMOKZvk02KMr7LdHpLIA/He3H53S73sl09CsM4sPCvuW5a77zX1GF8BmMBiBFCDQzQ5gVwBed2Wn+Xoh8i2v39MkwAMOqL1ZDqzYoKVNjaLjzmgQlIUwdbrBNvk+l0rnGYsEhIXuf6ynbiCSfrcLEZ1q5lHMm2nmoZHTMBdzFiYB0kM9rtE+5A7oiGqNFiMCmXsN4ukOdi9BxoSmSvrntV9FMOD9dDvsyBJ58FB/EWNG86YJPyPKge8EyEnNar+j4HkfQrln2oZvh11drlJF27DrDLFMWUjIOe0cR5fx4R6FODA9GeiB5NO/HkkzTzN9PRYUcdeaTttNNO1tPX3R4Y7kqOrrAiyaTApKKGzhfrRUhOjXfzpk1215136TPpu013dtipp51m3QFJFkmkUhZar30TniPfJ3Xk2jXcjH+Des95rZ9zgKFiD3leDUCFk4K1GAbOC/Nwud3EA3dcJsojJxpuKDeAu0cWJOorp3KO+gmc0OCshHR1N27a0EZVyXFiWURsF3ltzyPwOIrnO+kzdI1eNTGEw0CeGRHJUpEDX7Mli4Zt84YRm5vdauOTs3bvvT9tP5xyuWp7772nHfaxw6ze9HoX/7FZCMuY4aoQE5YLigK1mnIxQDVm4fJvroNNBljGgWKxObBYOsIn1mNqhnqnayBJlLVWdyudzcmy4528tIO0aFZIdjx05Hnx4OKxly9f7p0mvB8Qf6BJ4pkIaeOsIG0+SeU43zcizK7cEL2ue1yMppfEvM3x0ssusWee/psNDw3bBRdeoNEVPDM3TOT/EPKZ7+O90GwqNjk/5PPTGTSavEykdchkbNPGTWp/5N7F2ir7xDoaBRSoi+hPf+yCDCoblmdPuqJul1Dj5hoAHbkeqJSF+TmRX1DHEPIaJkIQwRA5DQ8NCXhcvwH5UydOyFtlMup5Rs2T0JW1wuMT9vLzKOYAAozXQ9HigQcfsod+9ogM2qXf/KbLBNHvHO5ftfgwHV5chihC13R2mdawUbPpiUn79a9/bU//9W86H6z7hz9+qO3z2n3UZonDmhifCCG+r4sojxIYNI8GUQOhsSaodWjPMsKFXJq6c9DOis8+8ptFxAjMN13T3TevbmGtWCQW2vOJpoYUUfei5zXWkLiQqMHEQYSooIG+hK+0e6E5FVrAfMM0BSpA8BfPMnRBKLw2J4uzkbwe6nImWFAWESs0PTlhhblZK5Xm7bbb7rZKVfibVSo+OOsb3zhFdDwOaxQJw5qh37NkyVJHYTmkUTS7s9PDopBfOs3QD4NvXJ8WoMHeoS2O16vUoc4npEUyolYuFLGq3eoBFlraiSbTVtt9993VZM3G5UHwXhxOQs04yYADDW1TTRvULSs++TxeBwupxoXwwD1UJix1EXGiCnFnw5BoQDmMAtfOPbMx5a3D+BR+l++DTQCm0c5HLZV1Fxm/XcpquTHNuNfAC3JPIKWkHfybe6F5RCWJhBNhAFjEpAp1fg4kkQLrRkjLwfJIzCVvMBpEVj4LykeaqM85iBQqrcFwpJl052QYPoP8j+hN0R1zkZnDCzc6TLHHywoQE6vLa+UxR/aupAFhHOL6Jj2i9CgO0NEb1ON+EFspUHxZ73Jx3sZHJ+y7tzDNsKa1xSmccc5ZTv1U77VfZ+TCtWceg8oXCsr52UfqE9cUBFck4SC7Z3eBAHJ9DjYRC5x+rivyHhwHSVjiobvWtBgx6Vxkkmum0TWtkWhaZ65blpzFcGU/V8b3oUyIwvnsl7gQ0VuACBLqxFY9vPHM9LQsBt6GUDbb6eUUwh82EhcDOIQV5RB70/SCWtnoQnns8T/ZY394UkbEZ+Sm7MijjrDBoX4hdlh5HpZ6cxeg5rkFhjiBtYttW5EYTwjiuV9TVpVwn993BL03jNx0obFYp4RiSU9qXz96TS3lwrvtsbcOHR5WZZX+Pv2dz8SzsSasnTwmn1XzLpdVK1c6zTJwwHmAnuN67qoHRT4emGF8H91o7pPnAT4FRsD6z0xPel4ZIifPxXXc9Z6RfgrggVHEuCl/DZJDft39ogyKg02ZLvT9ToyPO5NIw5l9jIlyZJWTvJbKs2PzQaLh/VkDMaVk/NEYg0SQtgWV6FwelYMbc9Kx0VE5Dg6gpjdQmhTYWdckO3jU3DMeSyIMoP5SHWFmL9ex4OXHUGbhPRj+xvvEBhb2AmBoVJFgrahJO4EIMNJJ/eyL2C+LjpYbcP6vZi88/7L94Pt3qwIDR/6d//7vUgrxBhQOPVx+LyG5fDBytB5NxsgEOi1ALfsUI8nzi62ArHPkLHjakdbBxYjLS4f2V3ETCJVFPVOZxiVDlDMglVEs29DwYhvoHxRQ5cBEXhuG36EkRElk8eJFNiutWQcmWGSsI9aHkEYxOpZNbW8UkskvPPTBU+G1hUiHkYtxRg5Op1YuStFw3boNdv0Nt/iUd7G8Grb33rvbRz7yIb2/K/y5BUces1Aq6SG47AfKBt7xoQNLaBg6PVgMrtfRPY82+LtI5gAUoJa8V2fegZaBfk2B33XX3RQ2Tk3PCQySqBh0R4TGOjoEtmGQeChqN6tV1UWjqXP5vELNZ/72jHKZAw84UPegUDp4WylKkJMuLOi9d9xhB3l6CWnLmHhxHw9EM3zMg2K5iAcvFYlgnOJ98dxceSSmF5R+fKbt1PSEDrBqp8H7gETHLi5ycn4WW+AmJpiRO+RhNyywUKfGQzt1Mi0j6sQJBqF7PzHOAQQboIe1IqfdsGGD6I6sNXk/e2l+jqnvPhGANaDUFBsTiB4wPvGQz8/OKn9nXQX8BPJDYX7WwUPCZnAJOtF6eqwz12VbtgC+dqiZgc/j4PBzR++JLd248FVr1tTNdc7Z51kuS9NMwk77xhmWD2NGNGm+XlW6QN6q2Ukq73hzSCz7EYGgPY3zIv/n/tgPrFVspMfAqhRJpBRok3HvRr584kffu6yl0EXuOKML5hdgTnnu0KlGcw+38AqxgIzndC4mm4nQNr4P1mjRcCjF0PkfSNKx3snDQic5ItSEztyItxB6Us8NYZHYaAAuszMT9thjf7Bnnn4xdNI0RXE85fQTdYB4LxElFD7lrVh2Jg8v5nuIgvHwo1wOOTq1Xg8LfTQGm4tQ0nMl18OKXi+WTJRnZbPW09tnS5cst3Taa71bR0asp5/m7U5xlMmXyWy4Hx18wLLpGUH66vrIeWSAl1g0vEQlBUJRSQBpyIELsRNBM+aRtePhY4Q44MuXLW+XimZmp2XdOS3IikbVB5rGly1dai+++FJIKZhQx3QDrw1ivHRdMzNyy0ReAuXI18TbriospguM73GIQUmdUFO3gaFh27R5cyj7lLUPCGPj3CCfUuDaWy6iwExbryQAYIk1lUqqbs+9EplheOMeoPWPgyDEP5AyOEQYNcJhSRmFEk4k4uAE5DWpPde2TUXwkR5uuB3xzqkzCU8moCkSPJQmecSDSotmBYEnbBedUY3AmOy7776qj8f97Q0S6GA5b53rJudXX3Ag17A/XEklODmGdisF9W4wIpioxhFHjjhD0NMYnAlGIfGTO9fo4HJx3d1O78NS7LXn3vb8Cy/oge6wYpVYSngvXudzQJFc8Q6N+MEsLl/Qvcjv1LIU3o/F4CZk9aQ36zqxWCfek4VAw9fbmpyxFRX7CbXGx7bahvXr7ft3/lAaQlEB4evHHBXC4G7p82DRmE5OO5rCRw3faijnJcSL4SgbSXB+AHxY8CgSzsPn2tuatlGdMqh3gE4K/at5SEoIjbUXEIaIdtWjDv6LFpjPldxL0eVNRbHLddjmzVukErF8xY7aLNpMKEKE+jDX5F7B0Wz+zXpxSLhHDgossfiFCke0ypk0RsjRejYGUYd714ZyWIw1hjmG2Zo+MDCgtIEDTJjHsxDxXjUNJgV4OZDfLWqcqOsBA0Byb3wW6ChGgGtWjZRDgAcNhA48KgPbuA+tSSibOTjjmtwcYkTiXL+Mg+sbXDgAZSd1yczLK0rOt97QgQc3wdBzTzDhRIhI+GxaB5kQ6+/TKBLXE4tSMj6GlahQTkpcdMLcbc0RGB7Wjb0TcQOF0YFJxnPaHvCKZdLI6WfdYq3Pwc1SEJh3iSYdSPjQ0qqecVVNgW7cs5f0MEhCzR+860qhyiwKibv3vjKR28EPFp2DouFJRW9aj83vxP3KS4JiIIuANaSlTAJe0tXJtlvwonypfr/sdVEOKEgvB3ZoyBuL8XYuadKlG2GTzk5PaF7tj3/0sG3ZPBbqmGY777arfeLwwxXaU0cjFOfArVy5wjZsWK9Nz6FsAzZBYDqCZzzVqE9E2KoNWSyqiM5hZD0wHJLHIT+kuVoHOWGLFy1ViyH5Oxt+enZGeTqenPVkU4Im8wBZDyHdDdMDIb9y8GdE2lE77bqL6nkCVBLu1UFcIyuJa8IgRuSe94ujKXffbTd75dVX9bO48dXAX3HJVw4qa07aIo5w1TefRlqG8TNCzK0lMgThN0Z03br1Xr5iHAeT6oLgQQxdKzUIFA44Ue7ivdjYTmllH/kAa/YQeABGZK+99lLoSu1206bNttPOOwmEZG3Gx0Z10GNr5NLFi9spSFdPj6IRIhUiQYnei/bqbYkC7wK6z3uLRgn9NnQPRa9KAz7eGULN7KzvUT+8pAwdGvki2iRRaMajnGiQKOdg/FlDdSjh7cVDQD+cUlVJRhtjvXnzqK1cuTJQOSHpIEAxrOuNnykuROhVdnEAxoQ6YwyHE3W7uGfSCowv16gJgb+8/4YW4QCHgxonb4Rbh7/sOkD9No/anEYzFGzVyh1tdsZnp9CRwYIhrk1xmvchNCMEpMYWSQexw2Nqerpd3iCfYXH4fTY+D165cbeTGTAQgDx4CGiKauFutmzdulftttvucBCnRY9qhx1/8klqII+80wjD8x4Io0dubkQ9IwiBd+MhRBTVhejo/3UpUg1xDjNq2HRxTi6bVSGX6tg+uY3rQL9Xqn/kcINDAmswALxGiGc2o8OD1+JgIYvD/XPoXrvPaxXV8FpFMEGtYnJqQvcVw2hCcA4HXVQ8bCw4+S/q+9G74X0U7klQzdVFuKb43soP83ldM3+PKUZPb5cT+pFuEartSK84y4FPrWpCt0/Ac8wjpDZdcNgn9Yzo2WXTxUPFvbJxd911dxuiHFepSO+K+q16W2HepQEG5wOg6e2RFP4j7ZG1IzReuWKlHAHvzT6VMlGYmAgOgdGMaDH/pv6u2VdxhCXRkLrbnCQSw1KtF+iwaKeek1Ka4nDJmAZhAO4PcIn8Wg6ICEo9x3hoz42JbMi11WJIWhiINxxMqix8eQTgiDZRCgdWbYQouYSxrDHXJvVRjblU0rlQBPXgXWs17JEfMmaDw0bdjgiSjckCLlqyRHmbtGeDcgULNzDg4SgL19MFAr0tN+OwKZfr7DSQSQ1SCiUPLG5nR05yJ5ETDMghS5JMS5+KjQ4QRrsgpG7lK3i+uXm77rrrbXYWhUGsedIOPfzjEvCW6DYHIoxu8PCfMNbHo/BweN+h4WFZbLeqHpoJYg9av5QuhCAX5uW9o6aUPGYYQA1pgXo03hgQig0/NDiszxCPWTNnMj5oOekcWWp47Y3AxMICD6JPv0+3kbScQyfPyJYtHq6LMeRDwvldlRSE+Pq/QUoxMG394qBqyIPm9zTLdnBQFhsSjUJfGSMvufAesSTV1+dT5CIUHRlw7A1KGD5Hx6fIybsDGs3O2dDwkM3NOrWU9+rp7fayYhN5Xu8K4lDw+0QNdOzgtdk7pA2sobqOJNnje5D1YCPLcBRLEmEgyuAZq2MLKSBCaqiFAQvBAPMzyCGUsYh+hhYt0s+5T/SkWb84PsSBwKbjECE9QpdK3lsaXdt0sajju2SS66ppRE44fHymIkzhDN4pxl5irSgDqsOuCX3WAau4jvw75tMKuSW4j8P0hvnwIByFl0H3MTgY5sRDP7i6hfWQNEkYzSE91xQ1NBdmLgdVR8KJHMoSaBgpHNqmESw1Wak0kB/5IKyYL0dPR/4QifiIzmFR2ORYEc89E6Ii8n3AF7yTwnb6GFWg9+6O9es22g033KiDy3Xstuce9qFDPqJDyesxJEIc1e/bLdYLv4vnhfmF5cMo4AWwum4pPWRSGCMFyW41PwvoYWg2k+rVweG9sRGaj3kb90hfaewI0XCpICbg1txRXB7qDkxKn5wUQo4n5GHKC4f6Kd7HqY88yEIbrYWUwOt5ba1GiOraw2xijMhee+8VaIJ0L3W258KqZS6Q3rlu5U9C3D2EjnnqwoJ3VLHhhgcHReoXaJn0/JTckL9v2rxJhwKjBm7B8xobnQhlvLyaNYi4IjhFXVec5Q5+5iAi98hhxejwM0UGAJzq06WcBxMqKfaW5GOQPgpD1+ANq8QVOMbq2qrVbXxivL1vqFZgOGhIUCkmcAqkpIEqxbR3v3H/S5a6QDkHgrlUQoMVBi+0CUYQhiKRBWejkmkcQK7JGa61jcHnekhz+LmrdlAtIAXyPNq7rIhgQZgH5ElVsgyCfP5zb1mNgC5nkjIlLlZ740d3rRWtQ+1wuS7beeedVfoZWjSsXIcL2mGH5QGE8lYpYnh1uaBYqLEPxOqeF7CAeEM+VCFVyXMCHfSG10yxtj5P1DWN8N5sNDYNrB/EswA7IDJQVuGiG1JzNL0nr6c7o1Bgoh+AQtbO+MYZIrqLtSUVDpBP71DR4jFZjsgAiRwAjyCu7rQ838hCtfPdCpVFZEDnCKUHmrYVevqBEmAQh35r4rlHJhIfQENYAu2ICvjDVWjOjJsGEj3eVifBsKAjrNqpwAlv0GdTC6lX3ZgGBxcOJ8Tj/nzQ1oz+zfswo5XrwZsJIBGxH86413H5TIgo5HYoNsS8LZZ9eE3cILxvDKnVgkcXF/cS7hFjEUE/nAI1WIwk1xvzY1InDoL6o1MeNRBOUm9n40oNEo9a8vk/UeKHtcX78W/xAIICKN+X5GqvixJiANmv/eIf0KGVs+npMBKF0SYFat2wAEuaOhDJPSDYqslLnZS+VkaXIL/TbHPlNYw9MLCoHEiONVQSeD93DC6JxLPCeVHFYE3c+Xj/bDrp2loe+XjXlzqFqLA0mzJSNLrwjIXgy3i7cCLVEkWPqFVmaOlzuVmBjkEuKvHLB2+R4A6bhXsBIMITkRuwkVhIwjLfbJ1SAwC5w7tJTKtUbBPzuSlp4LYSYhXFRgNyMg5k9KocRAe1PJ/i4rE6nrT78CbAEfIVvg/ZgfIU3tNDu5r97OGf22//91HrQHIllbArrrxKVpmNKzkSych4aB05tHgnrCpGBoOiujGjKygvhEK3y6Z6mYTP8oVPKa9nLbztzj0714HCh4d4zmwSQ4YGAwmm+b1E7xb7TGMvLNeJ9Wajq1QRuLh4FvIcrsU3LTK3PodJXNhSSd4KY8drXQYXxpnTL32WLlGE58saZyn03NUjMURisqWZBtEVpIjmJEbA+hMBqbc1tEy64FnSmXIqw3h+jXAbeSnXHUdv8nPqvoTD3mTviv+xOYBoTTKooUnC8zwP+1U7DyguOTTeFnIPa+NtkhhJclTPodk33BBRCOg6ObaDe3QU1WS8aN8B5+AzyIcxBtKRAmkuV6T0GLEWFhjPiuHmnoeGFjkmQVQSJivKgIeZPy5BhFekf91VXSI4mWx5muYgYsL7xoOqpXdlIcjrdWM8qWYFB/4An+FVAxp0vOEj7jHuT/nxQ/ddL7E4z0e7xOkdGxu3WsOJ2yIwQE0MdDo+Tq9PJsRo0thCrAxhRo55sj4NnA3FwWEB8b54Bw4zG4mDy8YUZznr8iLcdERteS/4qBw0DozXZZ0YEnPVjRs326233i7k9JjjjrVddtlVjeNC5BAOr1fbmyl2qAA++ThFZ1nxYGP5ieuIvN/22Azau4LeMg8ecA1LiYohm5V71EYMetLx4Ea1CZVUAuvMx3e4mrD3ETPn1g0J60kTOgc41lEVSqK0wcMLYlAYMgwe+RiHjlyIPx008zICmxEPhFHU7FhULTTp3SsHkSnkNUyPZvh81oH1xVizB+L0PDWHMMAKemAq6XOLNMmgU5I2KtWNjyvSYLOxyblXZxOlbMuWrerUIvrBA0stRU0DaJI5zZAv1oTDzwaPVY5i2BdqGYRFFsp9tMPhXFTTDFPsYmTDtXmNtyED5IJ0/t5DADtoVhtig56i8bkcGtZIrZkBp2GfsK54eYXqQfVF7LpZF4Gjvc6li51Drbp0ULFs1pqqKAiwQygiGHAZIZyPKMNet5ZHDdROno83y4Qh5DRjhDWKfdPKoX96zzWt6HUAZXbccUcb2Tqi0JTNIIQxlWz3XjLyA2CGDqKF4pysOUAPelIuPpYSUBU5n4wSwUqSH/T2+CK0lQdCH6iG+DYa2qSEyVE931vtAHdQcHBBMy92t5x9AxId6m5sLLV0wX2t1qT4wKaK6vn8HpswCrv7FDQPPWMdWy1dMLNc9E/DpllUQhgOY+Qts/h4bTa99KBD0ZwSmvjWGtTkuk78G29AOAuiypsARsVGc1BJDAgglk809IZuNj2bAiPjh5v8qEMgDcCLG9WGjElku4iGlAAABCRJREFUHLkAuAOCfPEMYo/00CDtmgsqW6E7heFRvbzF5s+rrEGP7Z577hk4z82gPwUN1u9TG0rDnV1vC8EC38hzWicOBJES3lLtckQIGRc6wGPCGHIUviBjHIEZ1p/35plyT55z+8wmx1JI0SDZZJ1LHTqzWF/RalvNNjEEZxD5zUSJpD7kwp6COKkldhdFAAjsAqOAB6fCwXrwGsqjXBdeE2A1aoJTHpXWVRgMx30IeAq4DYeUZxpZXdS1Fa1pjlVZxoQoTPsj7EsYdZLMRaww39XGROJ0DHCMOOlCketvH/quDi5vitQpC7t1ZKs2VqzR0sdIvsfDQrGdiyT/heaIM1CPJ8RtwBRCX+b3dNMSZ2pWANRyDm5SHov3jaJx5DtsClfLiKJrPkSMDaiQubAgYbeIytH4oOFJ2w2X8gHEAC/T4X2cYeJe3bVs1RQQCtqE+NLUCg8yymCqplz0MDpuEq6L0hSHlUNMjiTygggGSK24hCgbS/U2Sb26zjSGI67X0mXL9H1J0kr42r0NuIAMAZpcMnquWQyAETm/fJ+p6q5i6WU0hY9hDWJrIjZE94JiBV40IK4uyObPis/HoLjXHNc6iElWWNDrBdIlgkZX8BARVCRS4Nrd27nqSYyEmNTI+4JLKH+UtIxPvZDHWzTsQGMwyBHg4/f5OWGyWFuBcBCVDsWTDmJ/3D+godD08F4YONoo8fQu8ufKGbyXUsCQa1ZDjdm7pHwNJRUj3r3rb0e+tOeSTq4gxdH0yNCdBHYgrAE1yaCGKU4yfduhm4jzQmUF58L94d2JcjylcoFAOZogX4tmG/tAEj9MhdBEDAeAo5H2PdzlQnaP/eKOFofHSxcuw8ILyJvk7eBapn1GEMVyFCAJpTX/pVbWJlfTr3RnAy+YDRAI77CMsHxCfFM+uJeNF9viVOLo7fG2qqSDEIAFHAoWVaADjQ1dPdoIKpHUnZIWPRNWnwdFQo/VxJjMzdH0H8XcHBRjcxNe6nfDOA8PXbzkozpynkZ6R1Mlxr7dRAMvo3iow/vBPeazI9UzDiMTN3e7vC0CRmIJBfqjxAoS8KN9GBjvx4Fg8xEGUq/F8OEJvdifkPdQTTWQBoRkS8PJSxO8P/VRwMRRGq41+DuntVdOzGiZMJOHDeKAYU20RaIdZzT55uKwSQo1oL9+nWnV2+O+KFeK8q5qpaTPFK1r5u+EEFe17c5uB4OIiOgiChK6sfwTh8Lx3jxD1/XyWbWUsYg08Oisgat3NCSBxHvHvJjXy6BovCtRlbf04RBE+glD0/g7835cAgc8Jsw9qjnlF1AxVkD4GSArnpUDRB0XY6TSHNTgJFxjIifmCnmDCsqP8fBHYJFnuXLFCj+ImYwOL85DVMjQiKN6MEO0Z+eUQjr0FWq3lZKrcbAuoRWQn/1fbh9VCp+xIjgAAAAASUVORK5CYII="/>
+        <xdr:cNvPr id="19" name="AutoShape 9" descr="data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAO4AAACzCAYAAACO/iALAAAgAElEQVR4Xrx9B7hdZbH2u8ru/fRz0kkhjRBKaNKkKCjGC4JSBEVERLkowgURFDF0RQREpLeLqBBCk4RAekhIAukV0nN62b2t/j8z31rn7ES8/733+Z9/k8Np++y91re+mXnnnXdmSXNef8Lp7e5Fe9GE4QAOgIDfDwUOZEkGJCDoC6JarcI0TehWFY7j8MeUFgVnTWmE6VhQIYOebFkmbKsKwzDQ0NDAz7MsC/Tw/u6fvpZkSJLEz4Gj0v9g2zYcW4IMFTfe+Av4/VFEY1E0NdbhlJOOQ1fBxt7eEtq7OpHJZVCsaNDLVew90IlUfT1s00IoHIJuWDhQigDBekh+P2RVhRrwIxQOIxAI8HN8PgWKokDm07XhUxVIsiQ+w8GktjiuOi6C+qZ6xEbNgG6GseCD+Vi0aBG2t2eBUBKOraOqaTB1Gy8+di9kW8M11/0cPUUdtiNhZEzG9791DqyqiY1bt+Hj9Tthpy5AJpNGqi6BUqkMNaDDNC1IjgRHTmHbrl3QjT4E5ACi4QiGN4RRV59EPBFCa3Mr0uk0FFnB4pX7kSlbKJT3IKBYsPQOSHYJFcNAUFExcdp3MdDfiaOmTESxlMX0KWPhOEVEohYCko1oMoU33liBbNGHxi9+CTvrfbhg2hh8eKCI7v4sUqYExTIxkOuB0r8XqR1zsbXhHBx53NGYEMlj1iWnwDJN7Nu/B3975wN0ZDVojg+5ni7cdPU3UMz04Y677sT4YSMgWRZUWmjLgGQDsB1ICqCoKmRZAiwH9B/9oz1A14WvigLouoP2TAH5ShmmBfzp7p/g5OOnoVAoIBwK0VblPSY59Fwd5XIZjmTRbuKtJdF7ObTDh/ai7dA+Ez/zfk6f6eeSIiMcDvP7K5IC09Yw85qHUDT8fJ0cxwb9pzgWTEnBV49twN0/vxbxYZMB00CxWISq0N7y8fnRsRm6zucFiXaWeNDep9/9V49B+wAgyzKkt2Y/6WQyOWzp7Icl+wcNl1ZOoSdIEhTYkBUZlUqFl4CMk96IDDlabsdV5x4JRRGLrCgqLFODrmmQZBmpuno+SV4MOuBDFoh/DmnQcB1bGXqeA6z8cAU2bdiK5uZGdij19Sm+MJFkE/Z2Z7Bu01Y0NA3Hph17kC5U0DOQxojhI2HoVWiaDsu2sb8UhRRuhhwIwOdX4GeDDUP1+9h4fT4VqipDVRU4tskGK7MhO1AkCRObo/j+iTGkGlIIDTsaVc2PVatWYv7772NvXxGGGoVtGqgaOizdxnOPzEK6vwO/f/Ql7OrNYlgqjrOPGIZhbY3IZ4tI5/uxZ38Z2/om8xrGolFAlmCaVciSn51OxVSwcfsm6KXdCPr8GD/2KMiOAUmy+QOOBU3TeHNqcgTxpsNgWXnA1mDpWSRiQYwd1YrO9n3Il1vQ3t2JunAMra1taEj6AElzHYSDukQMjlXFTgf4bOJR8KlBfPmweuzsyaKnZKLvQDeGNw9HKGhDzqWRmXMPIufciExJw5cOT+LSGS1oSiaxp6MTj771MYJ2FkeGu1Ep5dE6Zhq6s2U8/sRTmDxmNMjiFIlOlyxTGJktkbMkw5XF9w6d39Cm5o2tSKjqNg4M5FA2DBiGg4WzH0V9IohSqYRQMDj4N2SIWqUCTdc/13A9I6H9WPtetYZLzkPx0f7ws+E65BYkBV/+3v0oa2T4Yi+zgbNhO/jzHRfijDPOBoJxGOUKBy+Z7Ef187nRg+zCJudSY7i1BsuOxwtiroNhh0bH4P6Ovpfefv1JJ58v4uOd7TDVAL+GLCu8ib03U9w/oMhpOxYdNUzLgmNr+NrkJIZFyogn42KtHREt6bmGaUJRfUgkkgd5udoFOtRwLZN9ED/f0DTMfvVVpJKNqEslEYtFodBx0YlJDjp7s9j2WSfijS3YsrMdhiWhUKqiohniojkO9GoVXVoEmq8eaigGf9CNsn4/G7DP73MdDtiAySh85IBUivw2VFnCqKSKH59aj1R9EuERx6JcVbFyxYf44IMF2NOf5WhuGQaqugbTsDHr5h9iTHMdHnr8FazcugvHjW9GW1TCKaedgo49e0ExoD9Xxd8WWFBVen8/VCXIjpIcBjmPiiFhX2cnejvXwjIKOGnGOZBs2gAWorEwTKMCmyKF4+CzzhyUSCtkjkwyRxafIotNSf98QN+BTWhJtMA2FYQiQQQDYcDRYBsSHLsMnz+AhrNPRldrAoVCGjNGDUMoGsauzl70lGRs+7QXMnQ0+YH4wt8j9MUfoGJJuPCYkbjy9DGQLBu7u7K4YUEPDi9uw1H6CoT9QG9vHn2ZAhas2o6Ro8bCJ8lQJQmGbcCxLMgOIKl05GDjJSPwHLzY3IT8FECVkC9q6C1VUKjo7NzWLnwRsDTouuH+rRtJbRvlUpn34OdFXEZ+9J/tHGS4nhF6hhSMhNiI6MOEhEy6iAtveAqGwZtUoEmpAtkOwIcy5j9/PUYefipk1YdiNjcYSQOBkIisAO/LweD1OSGWtnZt8KX3ONRw+ZjemvO0o5eKWLvzADKmD7Lih2QZcNjKIUI9LSihGItgnA4TCvyOhiObwzh5HCAbOi9sNJ6ETl7MMGFZNgxDh2QbUANRROMJOA4ZuwJIBrmHocgqy3ywtkUeTHhdOuAP3p2PSCSCRDKBcCQElY2JsQW/1qKFq2H7gkikUti4uw+VchWG7aBUqqJa1WHLEsqVKhw1ii6jHlI4igBB5HAIql+F3+eDSh8EiSWJoy5DZFlGKKjycRBSaw368NMzkkg2tiA+9hhUKj4sW74c8+fPx/6BAuxgHJZmo6iVYRs6rr7sApxwxOFYsHgNnn11EZriCqaODHO0PebICbBMA7v3d2PJOh0FNECFClMvwbIcyKqCgBJCsVpEpH4kdu1YhkppP5pSDYjF63DFhV9Gb18/PtvdiXK5gmAohO4BBUZwNPyqCsumjUZe20E0GkCpWOHXHejajrp4HVQEoUoyTNPgcwUIIZl8/kWninG3Xo3S/t2YOmk8DEXCZ305pNM6KrqCge5u+GIJNMx9APqkmdAiPtw+82hMa9QwqmUEdnXn8KNXNiNo5zHSOoDj5U0YGMhjIJfHkpWfYvSEKQio4Iir6yZff1Wha2ox5GenLLsGYVJEk1yoTNtFQrZcRW+2DMPUeS+u+eA52CahP7DToy/IGC3bQqVc4c8SuUk3Onohmd6XIPOhhusZI6dpcBBLJIZMyzbx4uyleOqN1bAc4VzYJmxyNgZGNIbxyu8vwvBJZwOOD6V8cdBYfX6K2oBj2xzMhgzXTQ9duHxoQKu1axGFh+C09I83nnEqpTJ2dfVhX7oMS/LxG9hsHAJPB/w+vrDk4WWJFkNGWyqMeuMA0rksdn66E0FJx29uvgQWG54wStMyYelVmI6Ozv1VTJwymhfRkil3FHBI5CQyDIMWmAxXZMtbt25BYSCD+vp6hCh/USWOtF6ebNkm/v73f6Bp+CjEonFs2NODTDqPctWA6g+gVNLhyDIqlOtUHKT9bZDDcTbcSCwK2afA7yeHJENRZAHTZN4f8PtUBH0y5/h0nC0RP244I4mG5mGIjjkKhhnCwoWL8N5789CZrcAKxmEbQKlcZHh03lkn47KZZ2PvgTRu+vXT6Ow4gNOPGQ6fz0HE7+CwEcOQTmexaUcPDuTGoqrpkNUgZN7EMmQfIQoTajCJYv9OdOzbgFhYR2NzE1qTEVxw/plYt+UA1n2yw82f4tjZVYaqhGHLIYEiZAWOJMPHMM2Hgd7dGBjYiqAPCPqTcBxy7WLj0LUNBANwNBNj/u1ctE6fhnFjD0PBtNGXTqO6rwOObaA9b0DzBeG89zSGn34xtvRm8eSPv4rprT7eFzs687j6r3uR8pvQynlM8OUxrOt9+FUFz85ejCOmTEDYrwjD1UwOQbQfac1p/RlJ0abgvUZG7RPBw6fCtG30pHNIlzQOCC1N9fjHK79DtaLB5/MJjOZyL/S3lNZxoIEFmwy4ZuMLwxWG5BmLB5+9/UVPD0Wjg7CVHOH1v3oaa3emYdrE8QjHQq9jyRK+f95R+PGVZyI54ijYugWtooljd1MA+to0DE7dPCjM8Nt9/N/y3H823DnPOJWyhmyxiNU79sEORGFYFixb5Ld0IsGg8Bj0vSzRgquQLLGABOvWbViHancGC5+5FgHFgcMeX/xtuWzh+p/9Du1dFVx2yRdxxcVnwaILpci8sLyIJkVb4U1sKCBHsmnTJs6bgsEgX1QLdBHEg55pWQbefON9JJtaEAiGsPVABu37OxGNJeFICvoHcgypOrr74PMFYDWMh5JoRDAkDJciLm1wzuE5n5XYcBWZ8hUJAT9BOkIHNlKqg1vOaURTywhExhwFywxj6bKlePfdd9FdqMLwxwEDKJbz0EwT08aNxi+u+y40M4CvXPgLZPN5HD0hiZZWP+pSKUhaGU31dVj38VrsTsexZdNmtI1s4Yt64EAHHQRikRjidcPR2DgRDQkL06fGMG5MC1paGtHc3IC/vTofjhlCT08X1m/egZIdQH/GRDCsMtqhTeVXJRBMI5YiHE2hr7sLo0c1YOP6tUzYsHGoAeYi/H4fZNmGKsVx5oP3IkBOLRhAbKAHxw68i5FNCV53XcvjP19ZiONPmoGGuhhOPOdCdGUqGDlsLLLpbmzZ1YXOTAk7uotoVVU0GxvwwdJ1eG/pGkyfNgXRoI8Nlxy1iFoUBhzeD2KPkVEIo5JlkfcyWaXI6BzIoj9fheRYOOWkGXj0rh+jWCrD7w+IvUEGBQeWaaFULonXc0R6d6jhEkT3jJQ+e8fiwXQ6nkAoJN6fSCjbxDeu/QP6SiK/pSAmILcKWSrh+TuvwCmnngwn2gSjXIKpCV6Hoq2XchInQScnzon28cGG6x1DbaStNeyDI+6cFxx6wXw+j1XbPkUBIZiuN6YX9zwhQUpeG9vkjc4naBv81rlcDls3rsG5R4zAb/59JkcpQ5ax89MO3HjLg6jqfui2jnAwgCsuOR0Xff1USGoYNhm4ZUM3CbbQK5Gx+HDf3ffAMmUR9RQFyUQCDY11aGltRENDHSCVGWqt3/AJLKsevkAIn3VkUawa0C0H+zu6caBzAGogiGgsgT3daQSaDkcw1oBgLMS5G0UYiqzkrdldsPHK7HRoC8mSLTavLCNoWbhjZhPaWtsQHX0MNDOMNWvWYM7rc9CercIORkDeqGIUoVdNtDbU475brmMS77SZ98ExMrju+2fh+GmT8Lc334Bsy5wv+n0h7O1K4d0P/go4Oh8T5dm6XmGSLxCIYerkmYDUjWggjRt/+h0E/UFOXwgmd3QeYPZ007Z+PDdnCzLp/TD1XjiWAZvRggk4ClQ5iFPP/A5WLF+EaUcchfXrP4Bl98Mh1FZDhKi06UMxfP+Rp2GnGnlNRvRvw5HlZYgEAwhHVISCIa4weGzvmKMvRFHycVWh78AO9H22ktezq6sH7fv70JctYf2eHDZs3I6Jk8chFgyCAAXBWK5a8FoLR885JuVvFCdti9MYj4El8NrZn0WuojH0v/m67+HbF5yOYqnAzp1gr8cq67qGarUi0JxrIl5kpc3PP6/Jb2ujrWcojDTDIjclY9MNA1/9wf2oaH7QVmXiSZahUOrns7Ds2e+jZdJpUKQQCoUBSA45UMtlpcXL0LWqfdQa7ucZa63RikA4hBCkd9940aGDIGZu+9792J2uIhiNI18sD7JYnD9wDkjQcsg7yQx3KQoDH320HAFNx7Lnr4NlG1i6aCneeH0V8mUdVd1kOFhiRs3Ed751Fi666GsMMYjrEnmKgObLl67EiiUfApbId8jzOZaNUIDIJAXRqA/1jQVEo5R/qEjnYgj6QujOGXh35Qbsbe9DIhLD2LFjEI4nsGnbLhzIO1CSwxCIxBCOBBGJEUnlRzDgd8+JclmBMCjvo+iryjaTPcQkRmQHd3ytwTXcY1Gq+PDJ2rWYM+d1dOU0WMEoHEtCSS/BMYCgLOHxe29lVHD2hQ8iFAihpa6Ec04ehzETJuAvr7yJdRu2wLJUnHHmJZj9+n/CsEqCA6B8T6GNHMDxx50GvZKCjh7kM/tw0w8vwbhxTcTxIxJOoFQsorOrHZt3FfHsnA5kB3bBrB6AY2XhEPPMgddBou4whCPHIp85gKOmTcWqVe/BsnshgQi8Wq9v4oSTvoThF14Ju60VMSqNZbM4r/wGI61EIopwKMjGRAZsWjZGH3UBuopVRPwhdO3ezIbbN9CPnp4+VMsWduzpRE5twOqVqzBlymTEwkE4xH0QQeVufoLSTKR5ZRoi3QjJ1+xmw7LRly8hUypRpQXP/PFOHDd1NEdWMlwRcYVD0DQqRwpy8vMMl1/ZEsTUoaUgj7kleO4nppqDlYWiqeC8q38LnegZm/JziqiCT2gIGnjz6evQNvF0SE4A+VwfVMnPTt/jZWzLYkL3f2O4IuqLGO2t0aDhUk6QzuexcnsHlGCEa4CcIzA8pg1NueAQeUAHRAYlfCYwMNCPLRu34sGffAUL5y3Fkg9XYFxTBD/4xnFQ/SYK2SoyuRIMUwGR180jx+O4U06FYzkwyP4p4beAmd+6FhWNDlCCTBfCshGNRhAKKQiHA8hmswxnJRAEUeD4FZx53CQcNnY8Hn7+TRxx9LEYPXo0ksk6xJIprPxkC95atBZWKI5gJIxwJIJQJIJwNDxouGSoDJU54eJ/8PuEU5HIcCUHv7mgCU2NTYiPPQ7lagCrV63C2++8jfZ0BXYoCttwUHEMmBUTsmXixT/ciXKphPMufwTZHHEGQJiIp7AFxwxCkoKgYF8fj2Lfnq0wtDwzxQ50Jl+IufzmhZdh4/pOpMv7EAr5UBeuw+XfPBqpxggTTMSyU2R55fXVeH89UEjvAcwydG0vR3AyWhkKxk8+DwN5BY6RxfRJh2P5h+8CKMD2nIVrNFSrnDrpTGRDEQw/YwaUxpGYFtfxZX0hfD4LwUAIkbB/kBfQdQvjZnwLOUuGrRnYtGoxunYsh2YYyGULyGbK2LanH+VwK3Zu24wxY0YgFgxAdmwYZAFknLbNXEPtw2aoLwgpLxoaFtBfKCNdKDCBOeeV32FMYx0q1QqCQQ8qi/JMuUxEnyhZ/k8MVxgpQXSZ0yjVI5UcG3MXr8Ksp5eCDNCrnBA/Qsjm3uvPw8wvTUW8ZSpMXYamFSDZxKGI8io9n2yJUqH/qeF6rPY/Ge4/3vxPhyhqgsvFQgGfbN6BPtvHxIa3aH7Fz19zHkJ5oELlIsG6eqUf2ZGxZuVHMHUDl55zLK6//EuM9Z1KN6qVKtKZNDID/TCrZfhVGUEiqIJRjD3meE726QA7duzGe6+/jkJRh6P4YYrsBrFoDMlEGLG6FJcT6PndPR0wDBnwJ5Cqi0GzVVSUKKKJBLPb4Vic2dLO3jR+9/SbgD8GNUL5bQzhWAThcMhllVXOuchz0jlRfsvVJoYmJp9zQJVw/8wWNDQ0InbYsdCrYaxavQJz352HfdkcDH8CtmGjajswqzpM28LLv/8115Kv+dmz2LSryMgkEkkg6Bfwj6KN6iM0YbIoISL72UkRdFdhcU5HHrp3YACSkub6X110AlQqwTJBSLyAhWRdmNnskjQM7fu3wC8XUCz0wrAKgK2zcGD4hLNRzNporIsjEVexaeMKhEMqKtVuEKwUD4KpKUyfei62bfsQM0b146YbLkYIKnxKnllbZuOJA3DJvELFwLgTr0C2VOVIt/wfrzGZVs7mkS1W0NWZRY8RQFaz0NXVh/EjmxFWVdiwYGhVvrYE+wXxKQzGE+uw3brf0/OqDtCbLqJUIi2BhGX/eAqRoALbMvm6kQPgNbFtlIqFQeKJN6kLj5l7oW9Z3OOWgtiwDgaq9BpUzQAhH0eBQSjxlqexp6sA2ySRzJABUgBe/vSPMGriZCjRNujEJrvkFeXe9CAcRdeb7clNTQQpO0QO1gCfwYMZKgV5PyI7ETm39ObsFxyCFSRWoGL+nvZubOvsgy2LNyXoKFFdlxhPiS4veUg/wxOCuLTZaAMR2bBl4yZolSoOqwvhtSdvhc8JsKF7LBoLZajUxAdNsMHi8o1eLsImn0BMo15BVTNQqlSYVKGLwlAl24mBgQHEQn7s7yshFG+CpgbQnzagBMjRCOaRVCrJVB0Un8rOiC7nDb9+FAgm4YvEEXYNl45fCC9UdiSKsF4mSjzhCUt7HKrrAg98vQ0tra2IjTkWphHC0qULMX/+BziQLUL3JWCbNsqmBVMTkeT5+38JvZLFc68sxe+feBeRSJyFDcKLEyynPFeFY5oIKn6komHOa5nIcCReg3JFY9hnoxO6pqOx8XD4fZQH+/nYy2XaNhZylSL8yeEY2SzhxceuRkXTUSxXUK7o+GxnN+56aCkG0n2ApaM+kYJjlZmIAqqQ5Cp8ATp1A4rUBFluxuYt7+DbX6jD5ecfjkgsCVkRiEt4NPcYAZR1C2OPvwIV00KxVMLcv7+AysBeFHI5FEoauruzqATq0ZMrsUOvT0QQpCgrO7BIrOJCR495ZUEEGZXjCHRHXArVYh0gW60inaf10LnKsXzuU7BM4gmEIkkwWsII8/ksfy/qwHSeLpHkGS7tWfd9DjZZfia/XiQcgUOGa0msirrkhkexr6cAIgYIGXqQmljy95+5EiMmnQpHjaCSyUNxlYB0DuyU4HD9VhyPeLBRDuLVQYL/0MNhJOgFULZHlx2X5rz6rENJM21yqn3mixUsWbcZlhzgheMnkkzQ3VSkcmEP5zgI+Ag2CW9JBrLr08/Q19OLsKNh5euPspqEuTPXy8jMwokDIWN0qKxNTsiWUJUcKJTbUCQmL6dbkH0+UViXJQSkAG6+6UZU8n24+LqfoOyQ2siBZDgwbR2VquYSHvQ3VI8G18wIkl13+28hh+rhT9QzxR8Mhxl+E5PKG4QgJW1OVomJTcPHLAlYpCoSfvf1VrS0CXLKskJYsngB3ps/HwcyZZihOi4BlHQTJknaHAe/vvZyjGprwPtLV2Pb7j5YpgPTcGCYFtIDWVTKOspGGZV8EX1d/ahLtXA9WcBHKtTTcx3ouoJYjMwzj0J+AKbhhyrH4Q/4och+2I4BWY1AbRiLpoiMvz75HT7eQECFLSnY9lka37thDnp79wOWiZCa4DTAz+UuujwCTdF7F/ImLFTRn/kYt1w0Aqee0IAEIRN/lEk7TmBk4jkEE7+/ewDTz7oWhaoBzaji5T/9AXapm6FqNl9BoWgiMmoSPtm8BZFgCFFFRpA2L103xxICCTcKUTpWy6p6m5UdmSQhU65iIEdSR4ed96I3/4iqriMYoDx0yHDpNSnieqUhQlK8prT3aiIuMc+f9/AMNxqNCqEk1YR1BZfd+Ai6shoss8yyXK+Oe1hLEK88eDlaJ30Ztiyjmi1wGsOkrquWMmxxrrXB/X9iuJ6he8fL8Pmtvz7mFHUHFc1EqVLm+tf6rbvQm69A9gVJzsIqHM5xVSFpZBgj0cUX5RQhxwJKxRK2bNkCx6jg2m+cjqu/PZNPwjPcIY9BjsuVmx2iYZZJ10nqIVa2uAbEb+hg9it/weN/fh533XcHjNgw2FSy4ryBlFyibkwPikZ0POSMtGoVT7/4KjbsLiLUkEQ0HkcoHkUoFB6MuMIjk6xTASlj6WvWzhJ5IQE+MtyZrWhqbER8wrHQ9QhWLF+MeXPfxd68ATuQYqOoUv1OE6TI+eecgW+ccQIKpSzLIelBx0JsOCl9mEF164tk6PRG9Ds6hXSuhFKxikymhP4BjevDp37xSPiUMhzbh3S6jIFsDh3tnejv70P7gQFkzDZEI3EMawghlYrA55PR2tKCiqni/cW96O7fCccwkAin4AuG4VcDzHIqfhlUDqRlLJd02DCRL27AQz8cj+mHUXpBjs67znSph67JrgM5TD/vGlimjWK+hNee+T0qxQFUqhbGTjsOXekqetJpLFm0GI119fCTcyZqjYVvQ/VMj3xhYyAipiYaUpAgdplUcgPFCkzHxsjmFN565bfQqkRaimqHZ+gkIS2XCoKpGvy5iHOsU2YbJ2XfwfmmZxQE+Wn/hUOkUVZgwkBH1wB+ePdsRnwCFVD1wWTE9Kurzsa3LzkewcYj4FRMvsYsgXRhMr2up0/mczvIWwwRg14Er/31obXbg3732aLHnb29Rezut3njFasV7GvvwNbdnZB8IRH1fKqraiHjpbrVkKqKYJuAKiKSbt68GVqpiIRcxtI5f+Z8YjDiuh5ILKJQYnkP78AlRXj0SqWKUHCoAE7L/OnmDdj+2R441QxajjyDYTY7VFcaR8ZApI4HgzivIK1y1wDuefSvCDc0ItXUiGA0zLU/IXEUOS0bK0dfCSrLBQnKCKilysAD5zWjrbUZ0XFHo1oNY/VHy/DevHnYla5CitTD0nQm2ei4CU20pSK49Yff4U0fDoawa+dOTJgwwd1gYv2IlffIBzoILoPQktimEMEwkqE6pMzFe8OgRg+dy0UiehuiZpnpQX9/Gc+9uQ29OQOmYXGEN9xIWjUIHSXQ17MTjlNAkIxXjUCrUp5HJQoiIKmgI0NS/SiV9uDF20/D+NFJ2E4RPjkoUiZeZ8GU0rGtWLMbX/nBr/jY8tk83n71JYwdfxiUUAP2dvShK92DXN8AlixchGQiCR81oxCooLV2RRdebuvVT739MFjjddFPX7aM/nyJhUGXnv8V3HzdRdCqGsKhgGhIcAk24lM0rcycRa3hivRMyA5rm14OsiMBqhmxEdcgCmoGlq3Zitsee4+5Gk4XmVC2+PfL/3Ijho2bBCXQBD2X5+OgaxIIR8RLu6UkjiT/pE8eMtxDj8OzGc5na0p23jlJBz563jF1DX35Cj7emUah6iCdyWL+ivUccYPRCBM0JLimjU1Cf853yB+RMscnch6XHUdXVxf6OjqhOCbef+5OJBNDxudBB2G4Q5GYWEQG0czqEsRwFVI1EZeEGUYpi83bd2Dz8vcx6ezLYHXUJFMAACAASURBVPBJUQRwSTJaJK/7ggorlMsYJgbyBfzi3mcRbx2OaF2Kz4maC7zcypPZ0XmyGGDw/BQu0RCsu/9rTRg9ciRCY46EpoU54r4/fz72EHwKJOAYJkxHZpaXan7JgIQ/zroVlmPAJ5G4YUhg4F0kigCs2GLn4fHzDovumRxwyJS5rUUoXQm9sEMhdyK6ZugfEWoWlW4klXQg/HeGabNm2zaqLM4nKSqRYNVSFoZEsLiC9EAOezu6kM0UOOqWKsQtqKhWC/jWKXG8P+99zDh6HGZMG80IhYT8JjU60DEDWPnxAZx79W0swunuzaC/vweFqo5cOodcMY2O9g6EQ1H85aWX0NjQCNU2IdN6knF45Tc6drd6QYdeK4Qg02NVFEHlos51XEcGXnriARw5vomjG9dwXcUUfSaexrJ0l032IrFbu/1vGq7fJ8qEkC2YtoSb73oKyzb3uVSpyzzDZqJxyTM/RPO00yHbPpQyGVfCiaGI6xmue9H/VcT9rwyXt8AhjQdS18fPObRYtOGrpo+VL5v3prFu2y7s39cH+AMIx2MsESTjJT0sRWF6iIglDI2pcdvi1/ls+6dQZRU/vexMXPJ1OinKlwnGDhmrp0cm+BFPJoSHYwvyNjA1wAgWTexFyqJlzJ07B5n2Tkw45Rw4VhimQmSGDcu9eBRlCS6JPFo0O1DB/me/fBRGOIamEcMQikcQcoUMg4ZDqQBLHsWmFBFRgiXb3NJ298xWjB09AuEx01GtBLB6xVLMmzcXOzMGrHAKEhFTJCYheK5pXPp56r5bQfXH715/G0cs4glCQT87wNbWZoxoSDDhNXrkKIwZ2YqoP8A1cDIM3ZLhc0j2Jwg6Ph9Sj7kX0HbIcAf7MYauO62fJNaktsBPZQvO+zjrcL04i23JH4jfkbabriWhDSLk6BpRC55qmUyO5fJZVKv9qGplDPQPoFx2cNzZX2NisrtvAPs7u1Es6yiVirh71p24+qrvQfUF8ecn/oTmVAphejOviUWRmARkVEHOyJXUkiKJzlE0CIhcmn6fq5jozeYhOwoWvfkEEhH6W2ouoDyf64lMDlCLH8Nk9yJSXsuojzMqcf619dta4sczEHLqvC9ISGRZOOfKXyNTFRGU9xqhMBs48eiRePRX30DzmJPZWZZzOf47Nno3paS9eBCa+Dz6mI/YhfPu9R00VBdJ/JPh9qx9zuFNQR+mwdEiW5Tw8ltLMHflTij+CKYeMRWf7t7JjCiRIvFEwu388fpYRZMAlQmohW/7th1wDBtNEQPzXvoDQyPR4TDkOTyIS9G2kM8jmUzyoVMOzZSW46CQLyIeF0JvWi5SAX3w/tuIROphGjpCreNgugw7HT/lJ/T+XnGcFo3E9ER0zfr9k+gqSmgaORzxVJKZcc9ZeGQURVeVWC3PcCUZlmTB7zi4a2YLRo9oRZSaDMoBrFy2CMuWLsG2vhLscB1V/hmmizyWmiscPP+72/nrS39yp7thCaEIpRZvGHdN6Ou2hA8NkoWpk4dh1cZdWLlhL8PJUDiCYCiISCSKRDSIQCCIRDyBpsYYhg1r4xbG1sYGpJJ13FssSSoz5HTuEtUy3dqhR76xQTuUR4quE2om4fXmHlEPFdB5O1AcarhQBGHIcJqgtIyqVmFij6A2VBO2IWNfVxe6+tP4aNUneO312bANDTffdBP6+3vx1OOPY1hTI/ykTnG9DfEGQn0lHlTjpPIdOW4my0g1xShMkIx9uQryFdGK+MmilyGZFShqDVJhMYWNfD7nGq0LlV3iiq6HMLyDO4J4b7lr5BkHrTedK4lhDEvGGd+dhXKV0Jd4DVuiNhsVd/zwbFx20ZkIN4yFSalShbgCWxBmruGSymwI9oqU8vOgb609H8QJHWLQ3jlI3Wufc1jVQUl9tYJqoYRyWYM/FMK2/Xk89dpyDBQM9pWkJgmwiCHMOk7aeNSWJgQMChe96U07O3tQGMjCp1pY8Oz9iEXpovs5EngH5RkuEyQ2XRyDI5JFulmfn3Nq5ni9xaJo4/jQ3bkX/fkydm9ajZYjzxyMtMK43UK3y1YK2EzG6+D1eQuxYOVOJFuaUNfUyAV20pF6UkfBIjtsuF7E5RYz2YbPtnDXzFa0NjcgNeE4VCp+LF0wHx9/vAbb+8qoqFGGoQTNqfZaJYG76eCZ+3/O8r6LfnzbIISSub9TkGEE8/lC2DaSYRWtsoEjp47Avo5+zFmynZ0T9YN6qICCKUUkyqGI9PM0s9Tw7UUpLyrQavgUkatFImE0NqQYriYScSSjIaTqUtxumYzFEIvFOHWIxeO8JtTU4VeE9JMdEkdwj+Bh+o6dA8H1bDqNluYWbPp0N554+jms3bAJDl1Ho4o7br8N27ZswquvvIyWBNXgqZ9Y1GoDPoEk+HjdmjStH7XwCQZYlCJFLyzQNZBHUTOYEP1o/vOQjLLYI16KQa2mBkX7koAKnsqo1nBrIm4tS1RruLSOdP7CoE109ORx/o1PcJ3eg/EWCBWpWP7cjzFuygxYviiMcoEbTTyZI+nl6UFk72AmSzmuLerTtQ/vfL2f/bcMd/+KPxEi4YdR1bFly3a8N28Bxo87DKPHjMawMRPw47teQqYE7vUkqSCdGBluMBxhY5aIbeacC5xzkLpp3/79fMA/Ou9YXHX5RXxBFDrhWqxu2kxsMJqxLCa+iBn2hyJQqNRUU+fyOEASDGzctAlrly3BUedezJMRmMgRtQpeOIKqBJmZpLIZ2GAgncGvH/pPxBobkWhqYQEGl7gIiioSZJUWlcK38PIcDchIZBM+W8JdRE61tSA1fgZKZRnL3p+LVavXYvuABiuU4IkOTAgZhhg4YFl4bNYtUEwDt9z3Z/RkM5AUHxziCwjNUsC1BFtvwIRP0jCtPogjp4xGb7aC5978EJIpwxcQm5PzYArBlN9S1CASjjeX2OS80VwJn5fzeaQdfab+Vc6YiQ+QHS7JGIZGrS01yjgfrx0Zu991xuxguEtM9GgHaQiBP4D6ZB3O+9oX8bVzzuXOrY/WbMQtd97HnUiU85KTvv7a72HHp9vw1uzZaEs1MO/Bx2I7/Pqe06RrRpvZg5W1ZKYjK9AtG129GU47Rgxvxtt/+Q0qJSAW9rP80/V+zN6S4bLc09Wcc7p1SOViMBi4TfC1RkTOgpvyGShLeOHV9/Gn11cy289+jI6VCSwdq1/5ORomnspcTyWbHyTwWPOgqLy3KXhw6Yd18Ac3FXhOdojfGGLHBc8zdGR8LWt+IA1seM5hNlbXUcxX8MxTL6OxoRnDRo/EmLZhqGuIY9GmDtz3xDuQFIJGAi4TbCZZoUyazlCAWUm6EMzYOQ727t3LTm101MHsJ+8REccRF0hAWfrWRrlY4uhBzoCen8lkEIklEIxEWEzheUPKYfkhAYvnz0NfxwFMOfVcFCkMeVDfERCRPjzDJa9Ji05tgNf/8hFE6pvQMKwN4UgMikr5uegM8vJIoVl2F4zgNxmu5eCu81oxavQIxMYdDa2iYvG8d/HhilXY3l+BE61zZXyUU5vCcG0Hs356FUa3NOOPL8/BstWrYMsqVEtlgo9guUGmJ6vQTAthWcdRDXFMmDiCHeRDz/+Dtdgh0vZSzsk1bTFKiNIL2XZQJa0vORzSWrmdVmy07ugfzyD4Z27nDDszlrDSMAoS0IhrQamDQQKYwcYSV3BB6YtM4htBlDGh5xKTV1xyAa64+Js8fGDhh6sx68E/uq14JGJx8Iv/uBaLFy7C/LlzUReOIEC6c76MDqgRj5w+oQeueXKaReIGKsWJJhbarDROSTMsdPWmWc134vHT8dSD16NUMhBx94zYFg5LTNlQXMP1Jmx4hisMxW2i9wQbNVZL78f1cR5mQCN1HPz0zpexbEs7p5GDdWbLxtknjsHDv/wWkqNPZMKwSow3iXWIq3GlkGS4hMC8CHuIQGvwnQ8yyEMY5IOjMPE2LvLJbX2BySnabO+8+Q5UuQ51qTo0NNbDFwpg82cHcP8zc1G1FDhU5yRvTOof9kwRhBMxzsHIyOgARA0W6O7u5oVsifrw9K+u5KjI9UNipSUgGo3xpIlqucJCDhLMMyFB+YbqQyQaRyQWH4zQg4YLB8uWLMa6lcsx4+RTobSOdw2XAyRffJ6+4ZJUJPRnHbRZxX/85gk4RFANH44wvb9LFFHvKpdEXEb7nwzXBu76agtGjhmBxPhjoFf9WPju21i9ai229pdhBOJQJUIPYjIIQWXdsPGTb38dMyaPRyZbQUNTM9K9adh5TdSMKSKo1DoWgOyXIUdCiPooT7aglUrY2UNCBgtVU6AHypUo18vl85xH9/TleLJEe0+/iMLcpO2q0hiSDbW4MZrynCVbjnAAzE37RF02m80w++1FQYLBXjeKKgvikDckOW8yLknCz677ASaMaMPEw8finQUf4uGnX4SP5bEW/LKD6665DCsWLMHyZUsQ9QX4fD1HEXAFCpSymIYQt3qkIh2PcPBMx6GiG+jtz3EU+/bFM3HzNTNR1g0WdXgEHO2bcqkoXqPGcAUUo2d5wp/Pr9+y8R9quKaG83/0IPZnqCwn1pgexN4/8ZuLcNYpM6A2jGGZq1UlfbkhpJL0jrKCSrksGHhP5lgb2mu+/l8Zbn778w7pL++5/wW8/e4KDBsxAsNHDceo4cNxoLMf+3uK2NbeCVtW+KIodAFcrSoVmSPxGM9v8gfDorOGk3qHHUFPdzeSQQkfPHsPbMliVRItABmKbFqsaiKpXDAYQi6bY8KDapBkzOTZQ3XxQXKKYBLlN8Qi9nbux89vuRNnnDAV4864EIZFr0ksJHlKmwk2ryzkko28TE+/8Ddsas+jeVgbQvEEvx9BP4uQgNuT662ngDZMSPLgr/vPH4GRo4YhMeEYWEYY8956Ax+vXoGt3QbMcCM3mlN5SjZp7EwVti5h5qnH4vvnX4AVb6yAUwoCVZlzZtpcZCB0Tixo55IHnR8RQRThCOoR/Ddg+2zOP4WWmPo7FQSDVJ5z4A8HEIyFEUiFsD+Txe33PIS8prNEj6SlXFvnHI+rbKJBnZwas/Ui33JkEdm8/lJO9bnrRaAdzxnTurBTptKd4/Da3XHzDTj6iIkMHd+evwRP/OVVhtMUxJsSUXz11OlY+/HH2LB2PYJcTpShGzpHVR/X60UE95AaiVeYnPTQFaVQZABVA725PA8l/OOsn+L0Lxwp8uRAYIgDsSwUC0U3PxZSVeq59R4eKTXYDcQ0sxuBuaVU5J5iOJxIOyi9+MJl93KrKOfhruHSMS5+7mqMnzIDUrAeWqHE50TP4sDE7fsSpx2i1Hew0MJzEt7hfR6z/S9sfPDHUvXT55y5763Ev9/2AoupKUeh1q2pkw9HS0s90vkC1mzeD43ADeWDPClClDaUQICVSKQLDoQifNG8aXZ0pvv374Nk6Vjy1z8ipGgiMfdOQhKb1svHPAhAhMoQC1fjHW1R5qHSzorly3Hdzb/FT751Oo6d+R2Y/DomLEkIKMhw6XUJ/hNbyR0dkoRVn2zCy2+vQF1bC5INjbzIPJrHJ5RankzNg3MEKemYKZreM3MYWtqa0DjpOJhGBAvmvoOVHy7Fp/02KoEUyztpjpJtUS23jEkjm3HzpZdh3RvbAY2YclETpjYh0oYzqefIfHykt5Vk6h7REQ7T0DOFCTUOiyYpcUSDB8kYaepAMhV1yxIWSw2jagRGtIopZxyFWY8/g4+27WSBfG03CoEKWj/elK7x0eant6G1EnBSEEJ8XWzRTMAbj8tFYs8QLPSuz32/+jnK2T5MnTIZr89diL+/+wEjCVru8SNacfnXT8Pzz7yET7dtd6cdSowcOGq5wgpKkYiNp23BbLw0NErHF6TyGJAt0IA9mthoYuHrT6AhKdrtvPRGnJOFQp5KQaJ0WGu43kA4z0AEXBaKO36+a7i0CNFIlH9GFQq6Zid88ze8LqTY8gw97lex5C8/Qtv40+D4fKikxXyp2mkX5JQ5fXHX1tM+1BqpZ7i15NihxNW/MmBp2Su3OFde9yDyGimEZCYe2lobcMrRk3iwmq364QvH8dr7a9BbKHGbmOclZV+Ap0n4AoIkYMKHciDyzI6Dgf5+lkGed8LhuO36K+AjscQgoyY2iPA+okDueSLvYD3HK57nMXE22tv34BvfvAbTx7Xhmlt+BZ17dkm44P6lI+qAJOwW8Fv0QqYzRcx69BWE6+rRNLyNaXuewkc1atfzC9gp4JXQVVPwMznitrQ2oXHKcTC1MFYuXYxFC+ZhR7+Dii/J4nMGfJaEEfUR3Pbti/HRq7tgFkUOGQj6xEhP+nAlo0Q8eudNAwQo76Q6L11sPmYaWkDjarlPlyZOAtEYjZMFR1yCspSn+ijXI8Y1KWPy2VPx7VvvwYBG8sCh+UbE6guyina5KMsI4cOQ4MTLY4XAwpW2shELldbQtRLr/PA9v0ZDjByNjRf+/hYWrFrLLXqaZmHG1HE4dnwTZv99Dtr3HWBDpbDvGS5BbZYzqpRiiYkSwjG7cJRQCKES20auUEKupENyNHyy6BVItu6W1Ya2NeWTNCBOMLT/O8Ol4yFy1TPcVWs34fr732HeghpYvP35hSOH47l7L0F8xKlcS9bpfWlAn6dFIHmrSeo1IumGorln+IP72/3if2W4k+plJ1bXgC9+4Rg4RgnTp00k14yq6SBXtWlOAwb6s+guaDyKdOeefWxwXLLx+ZmcolojDdCicgIzj/4Q1wdtW0NfewciUgVvPv8gE0FM8HMvgVvXPUQV4m0e3l9eXZFgGsE+0gvQTCgHWLhkCSKxJvitPIxYC0945KYFd6Eo36CckDuEXM9Hxv+TXzwEX2Mbho8YjmA4yOdBPoGIEq/vWLDUohyiSQ58hom7LzoMI5rqUTftJOiVANZ+9BEWzn8T2/pMlH0pvgQ0toZkfU/+8iZ8/NxWaBoxzIQ0bC6zcOSndjIvV/IJFpfbJCUbdXV17pwkMQ1C6GIN1j+LlkMH8XgMlk11VAWBEMEym6NDPBbj802NjmDBgd14fv57sG0xVpSWmssr7tpQV5qAx+I9BvNaYtTd60ENDExCsx5UuDF+rivYp/N9+sFZcHSaNAG8+tpbkEJ+TrF6OjswvDGJpvoEfn//b5FnKEkbW+FZw/Q63JVFY13IoN3ha8KovZxQ1JlpDwxkcihrxIWo+Gj+02wQYkqlkImSsWpahT9c6onhA0NlrwTEsF8Qp0OBwav1iqBAxBR1X9GDHP3jL76J1xbsQKFcAKwAbNlkNv61h67FscdMgD85Fk5Fh6bTNXZ4TJD30Fwya8i1eNLcg37C3zDicaW7tbCaf1ejiqwNbtKcP1ztkGiaCu0GVNauHujoga7ZKJky9nb2oaw7rKSq2DTWRjBn9EGGq6gBxIJ+qEEFpxw1FVde+k2ESSjg2AhbNBhbiMp9chWmFOA+U8mnwMewzGVwCeKSQoa6gOhCuJGBUz3RwgKLSjMUIcgzWxYWLFqAYWOmYNeH8zDsuLOhSTSYusYDmyayuRzDZc9Tkme/7Z4nUA7GMWLkaFAHCJezaLIjf/YQgDsilORq1MZoO7j3orFoa0iiftoXYBphrF25EgveewObe6ooqUneQCSPu/obZyHVIyP7qYlSucqCAsMUxkuOiyINPTjHNbwoJiEeCXInlBeNvc1D5JpHuCXjMU4JyJ0GAz6efEnMeLVSQoqN3kSmUsLEfzsa377pTuhOCTppi60AoBK7Keqi7nivwfzVy8Pcyq1YRMo/XRGBt6qsK3bHzNC1ePHRB2BrJRSLZWzftBWG5GDNqtVYvGQRfnv3HQgHZNx5xywUCmVGNz6/yoorehApRVM0BFkl1EZUyqFUyHuwZlxR0dPXD003MWXiSLz69F3Mi4TDBGlpWJs324wcgilKYm4XEIsuXMOlTb9h/TpMm3bEQWUVNg4XzRGxJMnuPClbwm33PI61e3X0pwfAzs6h62di9as3oXX8VEi+ZlRI8OEesme4jPZchOIZJn3mFKTWbt0KL5eL3K//leHWlvj4er36++87FhtjgJVi5Dn27e6AIUnoyVXQmymhL51Dpmqhq68Cw5U4EsQhsqohGcEDt/07Jg9vwd63lwArt8Ha1wt/XueezwANOKeD9lE+R80lshj9SkO8KJ+iIrwfMGmjBP2QkwnIflUoelQHKs2Goo9kDJFTj4D/xEkw+srYsHktwnWjsP69VzDpnEsZFnq5G60NeW+PiRWmT9vDwux5q/Hemk1oGzGKFUgEjRSfYDC9uVre2tJikkMIeIbbmELd1BNg6mFs/PhjLHhvDnamHfRVfUKcDgOP3HwjPvnLVlRKVGKzWMNt2SROFwNzPWUWXUSv3jxy5EhUCrlBgTvls94xm6YYek5N/HpViOdlVTjPaJTywypSdcnBUgV1Ek09ZxLmrpiD9dv3Y8n2PiarPJKJ2dqaAfRetBUbuGYSBXEQg/ppsSJkFKyTdpveX/rjA7D1Mk+szAwMoKOrk88zFg6jpS4KSyvil7fP4rtJ0GtRbu85K1p3ym+pU4rgMR0Hiyeo1cF1oMQ/6DbQl0nD0B185/Kv4hfXfpMHG0YOMdx8ITvUEfQvDJfSD683t9Z+PMOlVk8aLEc5r20pePiZv2Lemg4eAqFTSc5S0NIUxBtPXoPh40+GLIdRztH7esMlxFBFRnsui+8FDe/9/p8Z7uyHrnXIQ9BG4EWVVOzZdwCmRcJuDbmygWLFRJpu79GZRbEsBpEFVBUTxw7HCw/fgX1Pv4ny3xahmVhTy4JORjkIwQTsYxKopuOfvCNdZN44rs5YnKSASsK7C29Kt5fgMpSiwnfTv+HTrn6EfQ4yMw5D+7r1GDZlBhNUVCIgppE2vUZif53GwIioxqUMy0KuVMHb7y+FJgW4XzUQDKNAYgYSRih+FsE7sg+qTBuUDIhezcZvvzkWTfVRNE05EbZUh/WrV2DJe+8gmQihLpnk3tipRx2PHSvzyO2qwqLSEOU5VCs1RR5JkNbP6guX3TVNtLQ0CSTh2Oxo+JYo7JldNVu5xHJH2uRapcxaZuqljYSo3kjGX0HbyGZRBnFhV3B4ECt2LcTuvQfwzpo96Ncs+AjNhEOIRxJC8caQkGCP28pI8kFXqebVK72OILIjFnCwkIPKLQ6CqowXH3mAO2b6+vtQyOYRjkaQyWZQLlcxpq0J+YF2/OK2X0ORKbISchDQnPy2SlDf7+e/p3Wn1ITOn3N5cuZUEqJJoLaEvv40qo6DR2b9BF8+7Rh2eMGggMrMHtLAwkKW0wbBJAvz8FhxL+p58s9ao6WrSyiSrg8TU44Kw67wbO47H/or2vsr2LW/B5aj8nD1S75yLG7/0SmoG3MG5+Ua1W9twfyzU3RJtiFmXPSY/1cPdqo1TvJfTcPwXoMj7mtkuG4uyPS17EOpoqE/W4AkB1Ck5vqSxl0fNB7m48274TgBtKYCeOflx7Duhvswav2AgIPEvhEb546uZKke3cbD1aSqzpDQgVQ7NNWQ8z2X5fS8E0FKEmnwybh9v2yQkoRqQxSNc+7GppN/BPX2i4Axw5Hfvxtm8yguVYjiuchnaCN4zdqstWV9LDD71ddw5umn8t0HaPRJKOjjMo1m0R0GDOzsSGPSxAmY++EaaHKUZr3jwUsnobkuiuYpJ8FEEhvWrMSKRfMR9pNEzo94LIkTjzsHi17cDVu3eRC7ZwB0dwOumxKB4U7tp6maw0eMEPCONrM7eYGcZ5SYZWKp3aFq3NRNqYJOUjtKFQzWLVO0bWigCRWWmG9EghFqUE/5YLSZWL1yKd5euA4b9w3wZPdwUMW3vnwKlrz7Ks784pfwyYEBZKsO9FAYCo0gqelh5fUSN1Pi82eGlCWJVHqTEPH78Owf7uc17unpYeecLxTQ1d2Nhx55BM/+6VHk+vbhF7feCdumqZQElwNsUrTfAm5XD527lyKwcMaVzYpyM017BPr6M5xivf7sA5h8+HCXlRe3BiGWm4cdVopC6+TCYxaqHHrLm8EykyjveA9voiRBd3pNmvl1oL0X9z35Jj7d14dcmaoT1J0r49kHvoPTTjwCgYYpMGhyC6Eq13Dp9Qi91g49F4TgP5eDatllrmbUPudz8tpDI7f0/KzLxSBb1iJTKUblG2gRPCYIoWkmjwwp6TqyeQ37enqQyxmY/dxDwOLVCPz5A5gEAWkEDTUp0NhN13N7hjsoYXNv6ET9jjwS1VXI0KoMlYAczjW5W4T6GrmGKYkB5pA5V4r+6UbseOlNZHr7EPjFldi//D00nXAW3yFALIjDBundqMzzvASVaNPdcsvPccIJx2PSpMPF/Ct/kEtgsWgQYWJ/HQV2tYiySZMdbGanT5/Wgrpk3DXcBDas+Qhrli/CivXb4Jg6vnPxZbD3R5DeJ6Zc8M3PPPUPRXSXLaVxK4Q+6urrheCdWt34njlDk0VMQ0MoFEChkEddHT1PRBVTozUTs7CIzIKkI5GMIOgXih+WDdo+FJw8Wk9qwfxF89DbX8Vjf5mHlrY6nHPSDMx56SWG64c3xlDvDyHZ1gC1uQmfFVR8mqEZxUIn7m0URkS0nu45UeHMr0i47gdX47ipdFcGEz09vdi1ZzdHm/vuvZcVXS8/+yTSvfvwy9tmQYy1IqcllHVkoH6/mJfNyIxHBymMSLgk5DLZPAbVtJGjMo9s4aN5LyEcIsmoGBzvGS7fQ6laEvk3BQ33TgS1UY73xb8wXO6G4vsECRRChjd37hK8OG8j9nVmeFwxlaLojhMfzv4ZRh52JJxQGyoDNClTnINXU6Zq7v8Xw33lge+x4Yq8hXprxaym3nQO5SqVJGQUylWkswXIaoA1t+OGjcANV16GjsvvR7RiQyGFC3kaunuBIyLloMzLrft5bCVtANq4NLOYWU0yWpe1pIgkanOiBhbwk5TSHSlDdxzg+wYpSI9MYuLDt2Ddt29F7398Ax2fzMek2LoysAAAIABJREFUf7uKo43nyUhKRyIQik7UIUQRi2vQEnDnXb9DV15HXVMTR8CGRAz18SCSYYVvp0JN33UN9UiFowjTqBufgekTGpGIh9B8xMmw7QQ2rluDNSsXY9G6nShYPjzz61ux7m/dKBXLyJDTc7tQ2Ou7JVkel2LbSKXqWHBBtURyWNyd5IjeUxHZ6H44VdTVpcRgM3dig2hXFvmqblSQSoTgUwzWM5N6jYYDyLaN3lIZU86fgtmvv4RSuYx0sYot6z/D5s072KHQrVbaImGMTcV4cuaxXzoV7819F62NIxBuGY0NPT1or1AUUOD4ZKh0fUg3yt1TfvzsB5cj6VMwceokVj319vUxYqVzpTbNx558Cj+/+QYM9O3HnXfcC10n0YmQ/nksNZ83OW5XhEIbn/6eBBqeSILSpnK1yudAfMmmxX/lu2IQt1JL4hBTTQ0G5JQFiVMjruD+X1doUSv+rY24js2pCDsPEn0YOq6//XGs20OTN0WLKBXkaDTQ/Jd+hpbDz2SupjxAY3CH6rfEy/C0i0Nu3FVLDR+EAtzIKhx3zQG5XWMC4g9pGWoHWEh/++1VDrfEmeT5qa7mZ8Pt6s1y5KAhbDQXuT+b45IPlQN+c/vt2HjHn9DywU6YpHnlOaokCxNpB99gxKt7eY3i3GcpciVSp4joKHILL+IO1hm5Id5AmObluvI3rrdS2YRQgQ00Ln4YC069CvPVAdjTG3Hh1TdCc6EdvTcZiSB/dJEHsXqI2GMHn2zYiuf/PhfR+ibEUg2CuabJiQrBOIdvSiXRBShloCgmjhnbgu9fdBbqUjE0H3ESbDuJjevXYM2Kxfh0XzdOO/NsNJfqkN6pIJ8roFwSrX2skHLvS8T5tmEgHokxk025aTIZ5+dwq5/bZsdyTa2M+oY6Lp2EgwICewIVT95I+W00TPet0aD6RcSgzRcJBtGRLmL6t6bjuRcfxrixI3HLLb+FZft5YgjladFQGHU+H844+WjUtdRjf1c7OnbvQ8L2s6abjC+YiOPEiy7Gg6/MQzAURdhvY1RbIy788uloqY9C8ScwbORoXlO63SfZBMP8aASf7dzNDrF/oBsPP/QIHJvu9Eh3InRvRObuUS+F4uvqTj6hurSQPorNpBni9qWQqti46G9s2AG/qLXSg9YhmyVmlyg3t7zDrYuuJfDGHyrBHZpriroveE9yDm8RJ2Pi4usfxq7OLAcOErLQq/3HFWfh6kvP4NuMUJ+uWaSJk2Ltee9SfuuKfw5ihz8naWUU+N8w3EHKuqb1mt/v5fu+6/BoSy5TUKRUeeGyuQqqVBCn4rthIpMvolQ1MXnSWJzzxTORu+Be+Gn2DhkJyfP4s3gb2k6DD8/w3FGuRDTxIGxvzpNruLzQrsaWNi+RNNQB4w2sE2NT6bYaVHpSoc76Hna/+yFy23aj9ZEfYv3WPWgdNmJwSh95cjYe8uDuhAUSB5BEngaSjB03fLB5W6ObSeUK6M6W0NWdRldfBnu7+pGvVvkeMOefNAbnHjMKsViYDde04ti2eT1Wf7gIAUfCzAvOx5IX9kIrUBsXOQshuqCITw/asMSYUjtkJBgWEZSaHywDca59i6Mi50kbNx4VZZ5KpczrRPCVmFeqkVPkoteiOzqQzFNyKpAUMaKUcmES3g+UTEyaOQVXXn0F7rj1CqSifnSmy5g7bzXmv7+SeYgff/+7aO/eyY6G4N7WjVuRCIYRsiU0NTdg5NGHY/WWTxGoH43DRzYhEbIQRBWth02H7I/yPXubxxzG150MlwYIUB6bzmQwefIkrF+/ETt3bscbc+YMGi6thefQyWF7hjuIOujKMMnmZm+OhAoNNzctHHf8EXjmtz/jyZWkba9FdMQXsO/9XxouGSbde5mOg27fSRNGv/6jPyBfpuFwpA2gY7Uw+/fX4Jijj0CgfiLKxPBXqTQ3ZLgUlYX665Ce2/+HhkuWRXeZlF598FpupKc3oy4M2lQ0y4dCfpXuuseEEzGeOuh2nHfedgc+/vHvkPz4AE8CIHtj76HSd7X26pIbjsxMH32QekbIzWjciuhYGRwOxtIzMUCO2GfOrWoWgEem0hj0ACm5AnDO/wKkyeOw91ePY/z8h7Fk3SdIJhvEAdAxU47Jt9uk+7WIIWRC8yGc1D333I+jjp6Ok086Hg11CTTWJ1FXnxDsNwlFJBkawSTLwc6dW9EYqqIhlUDLEV+Aoddh+9Z1WL1yPoaNHoV4cSz6t1aRzZdFlGe45E53cNMB8mU08pNgqjhEGv0pBAGJRIJvjE2GTvXkFN2ylG+aJoyUYCRFFoL65XKBG0AYurqN5o5ThuqTEI8HEY0m0ZfRMe3iqbjm2h/jsDFNOPfLJ6AhKSPATRVRZLJVbNu6DTv3tKOvP8tD4j7dvoenbM78ytlwAg727tmBq666ENt2tKOkUeuljVR9MyLJVoTCCVSrJkYfPpmhPbVxljWhWuKvCwUcaN+PbZs2Ycvm7dCp0lDVuT3PKyV58lIBB4dKTN6m9/gBru3aDh741TU490snoFrSWdsucnBxl4F8IS+kmO72qyV+vNzW4z4+rxxE+zYaoRo5NTU4mLt4DX7z6LvMNg8y7ABWvfwTjJh8HORwI0okc3Tfj3TbTGqR2o3aVGv6bcV+d8VGh7TmHSSo+JyWv1qozOvi1oJFxL33KjEBgzYKTwChhmQaOGawbEvcmYzIFgmJRArf/NJMtF94F2waRVozlsNWRH7JCh0XpQjqX4Wf5zKTzlnh16U3pp5Nd6KS2MjEDjJcF1MXPCUJRyx3tArDKVlCOBZGaVwbmm7/HrZf9ksc9tjN2Ez3EyIn4d48igdeGyaKxQJveu735fooMc90v9ddKJbL2L51G49E0S3SvgYgwxT3DQqqmDZlIk6ZNh5/fOJpzLrpSjQ3pDBs+inQ9Th2bN2MtauX4vwLv4Flz+xFrreEStXkcyAvLfS34jYbDPdpNCmL4l1JHzU4KIpotKZzClJUtZBKxQdrpXSlquREDZ2b3akcFKF7tsrkBN2eYZ6aaBAlgngyiFisDgMZE0dcPBnfvfpqKJKFyy69iG9mXd8Q5FG4VIMncQSlPnmN7ujXiAULluGEk0/Axg2foLuvG3FVxxdPGEN3H8KBjjzau/qRaBwPNZhAQ0MzO+ymEaPYwZKx0qhUijYEZTPpAaxe8xHynb3YuHkr3+FBqw6Vg7xI6+X0XsSla13bm0vPo3SBHvNeewwtjUGYBh2vN2mSFFNVvpuBUOQdXCUV9wcWZsOTNEXB7J8EGCStJGfgkYWPvfgPvPTOBkZF3iMOA0te+wnaJn0JUMIopbOD+mRvj5Y1ocOujbiC63DFF4ccn2e4h+qTa2G21wLLebB7D2H++qW7r+S2Pmb73JDJ0xFNaimjmh01lBNDClxwwYXofOQt1C38DDrlIq5HooM16Z633niaGsMllVmMJt7R0bu1XVG3GpoEIFg4TzNLKllvSBqJ/N082O2fpIhLA7H1VAL1L9+ODedcj8SFZ0O+9DR0D4hiOF0fJr54lAz1xgqxN9s0T3OUEY/IaGtOusSYmJ5Bf5PJVZDO5LFp41b059I4bGQb/vzim3j+nmvQ3JBE27STYZhx7NiyFeEAsGdNHunPLKRzFaJAxYA6Zkf/D2vvAaZpWV6Pn6/X6X1mK2xhC8tSpCpNECkaRIiKKGpECEaTGFvswW6MiUaNvUTUGA3EgoogVXqRXVjY3ndnd/p8vb+/65z7eWaHDf5y/f/X7/PyYnd25pvvfd/nee77Pvc5567Okfp1QoZpZ2uSNz4Bps8Uk3MkChcf9aukLcqczpcRJC0Qqa+yHdFET5eZk0s2x7GjAmPYTuFxVEY6E0Z7Wx+mcy2sfc0qvOb1b0YrKOOyV1yGJYsXorMtivZsm2h7nekU0tl2RJKdQDiLeqiGZtWECZzAMDP6LKKFHRrSzLGos9UwxvPtGtZGVgkdL3sXLlHGwJqYLUQvp8zlpnHfA/cht/sANu/cgUKDtEBGbYciO902Nyb/L2TZtQx9EOF7Mf1n+s1rvP+2byOTpjcV+eVHjMHp4czD4k9tXLYIvcPin9q4HOotzrTQ8xre8nf/iKf3GxjnX9dceDw+9u7LkV50EoJGHNVC0Y1PcYMD6EzqpkL8v9y4mmPsAUy3cXXYf++mNyriCjmjEXeViCbnzhjTh1pWCr4TkTje+JprsO3PbkK8bJpXOdITTSYSKmd892JYd9pY/lwqEhNYpAfFDyHp3xEfKv4b00Iflf2pK8DfnTSKlVqknMERRSQbw/BvPo/Hzn87mh0pLP3Jx/HQkxvQ1dNv6bDT5Jar3LhszPOhW7pNjPCpDU/h/ocfxdmnrsXKFcegr7sDwwP9yKSSqFFTWq1g4zNbUC7PYt3q1Qg18+jMJDCy9iw0Wl04sHcvGjPAhtv2oVys2jDtqi1e/g4PRrGu5QHCF+VgbOewbJBDZjyqw6RULmHB8JD8kxlRBfTxMGUJ0mxq8bLO7ci2SeqXTFEfax4NYn9HCMxwpEkL3b19mKrVsOrCU3D1tdci3hHBxZdcgHQ8joHBfoyMDGrIeCKRFuHC6249+OWf/9jOBxCrjavGIb2QQpJqPYotB1tohNpxzHHLNN6kt7dfzp78OZFMmk3kCtMoju/ELT/7DfaMTgrc1CesmyeTRSXvV2aHz/ya1QcSUmp17dEQ7vvVv2jTUoTBA8Be5jEldJ4JqaslSRDxLUBRIqVNdlxheWs9v6+aITDFz84MslHD+W+8CYVGCKEmJ/MZ+v/Aj96PJccMItK1As2CaaT5rlEHlHnRvI+4z4/99mntoLXfPT+d9z8zF63n/bA3kfNtOZJTcrOzCH3rI1dr45oEyfSbQv9cjUV9bDVo4lWvuAKJ+3eg8tXfolzhsOqWLFcIHinyOlsSF/BslksohAy9mWnpwtS4BbFlJMTWyA9nq8oeYcvpK90GF6+TrQJ/ErOdIB1wBIloEvG2BAZ+83ncdcENiNbqOOHBr+MXv74DI4sWO8M/A6c0woMR3cnnWAs+/dSTeHb7dmzYM4njj1uJbCqJamEaq5cMYO2Kxdg4VsepKwdQZe3UKGKyGGDl0gH0ZuNYuO5MlMpJjO+dwYENeezeMIoarVnrAaanJ+eQZInznVuFZ+yQaMD0K0GATTrcCBrNGrq6utTKKJeL6t+ypBDKzxS/0cTM9AxGFow4ZRFRaLPaoVuj2mkRWoXS2qaB3v4+NDmlYVEPPvrJT2Dk2AGcfuaLsHb1Wov4PDCj1NqagyafA58/a+tcLq9NRET/0NbfIlKn/WkYyWQW1GLICxsxHJyOonvxaeju61Imtn379rk+KNfR4Z2PoDM+gV0Hm/i3798ubWpUm9D0snq2nPLoDmXeE3HfSXF06LsypGhcAN2CgR784gc3CYPpbOtA1fX9mYTRUZIZCEOB5y2bx7IbSSLFljNadwHK00l9nCFH2Ud6thbOvOp9qJEp1YqK/94KSnjsJ+/HwjUnI5TsQok+TgoqvOfmeOqHVv/fNq5tWPutz0Odj/r70a0h/71+MAFLE23cud5SyBrkmprt5nmSh3rM4mNwxZVXYfMVNyFxMI9yhDR3jdIzxY53p3cnmZQ1gdmhhOsEYQIEZAxxwyLkRNQEpqxtxF6ZqXNss1oqaVHba0G5+Yg0c1GlYmkk2xPo/eVn8ftXvxvZyRyO/f4HsTcGlDkpQJC86TvpFkG1E69ndO927N+9C3fe9RDOOvN0TWmgFLGcJjlhDdKNaTQD0h3LSKbiKFcpK2vg0FQZq5f0oTsTxcDKU/DcxlkUt7eQH6/g8MEpcGod20iVWlHSMtb+vB7W5MpmXJSx4VQ0SuNwZx5CQAeBKKlDGGHJ260jJZaYWfLQRYGqIbUbdMDVEI4Ekglq0gLR5gR7rsyLqiDvOdTfiX2FGRSbdSxdvQixBEn8hkgbG8oOQLHaHNWO6b1F2zqmp6dQ3H8vx32pHKBgX44VkhE20azk0X7shagkB+R8snXrVr0v21FMmw/veACHJ2Zw2gWvwdo1qzA4vEBYSaRhJRmvSxFOuAPlfkckfWSzsa7l8+PUP94bfvZjFmVRJZ+8JQs/A/doMkh2XIuHc1VMOO7XeqWEajGvsqXZpJj9+fFPQWWeoES2SS7D2bx9N66/6WaUajzsSSwKY2Aggd999Xr0rXopmmHSHE24ImN4d//oejL/PV8o4v6/2Li8Z3KO/M7HrtHG1eZl6sshRw1LPfggOX/0pLUnYnVyBOUP3IwCpVPhEKpEbclJ5hnujjAPIvHWZhNJoau68X6AsenEjEUTtsl4Qu2YsGmh+ka5a09pELmrizgtLm5NegNzsuj+wXtx/zv+CalDU0i94XzEr3gJDu4dg1YbT0oynypFjO7biX079+LB+x/FqaefiGUjWVSaKUw1ouiMtHDuRWcgGy9jyzM7EImnFfXa0hFUa0ChWcIdm7vwjj8/C0G1iR2PHEZ9KoI8J9FXgWKpigpBiQCoFHJz4BRjgJElzMmCC1GqKkaXaEz96I62jO6B0HUnvZODR7lk8j2SUFJ0Z3JSSNrjCHmvIx0nfZAHBAkSvCf8piqGhxei54xj8ehdz6J/ZSfifWkkmeqKceVSSPc8dLAgsFm3bEXVyzg0MYG9G+9DWyyHRCyJRNJ46VznTOtJ8avUm+heeQFqsS75aG3e+Chy4/tQL09r0PSrX38jhkaOweiuWVSmSqiXWwgaYSTCSQcSATVmbeQ/Wx9HBxEPEpZcYs0xatJ1UzOrbAazZYYE/VxfWzArwTb+n7RrJ1GMRhBLcqRpCBEePHTWFFehhuLMKAq5GTRKBi6RgJXiemlGNIPqi9/5OW69Z7MkmUrqQ3Vc/bK1+Id3X4u2hSehUamgXLaNKwsn53c2f+OKduvCuaXE89qj7utHR1wf/Y+Oxv77+F+uHw6RV6bCGtejwwTD6bzATgM3pdDRRh03/PW7cfDyT6I8OmGm300OZnD6xjDlbNbw9myYGNs54pG63N6hajYo2kHjpInF4oqOCTGirKbWAcKmN6ODU13we+gvNIe+hUNoT7Uh8aXr8dQX/gPRzXvRXLcIa778Hjzw8BPIUGGEFg7v24Otz23CHb/9LS6+5CL0t8WRbx8GFq3D7c8extKggPddPIxYiDV2BZs27UGUJIZ0CskUS4YYRpaegFhyKWrUunYPIRxJINQyMrwUILocuyamv6qtXKtCaKZzYWRWIeaXAqlzkaCG2PppcyNLXTFk0yO4aOmNWaphfHQc+zbsxaFdh5CtAbVWHQnqiNlWUx+9iXC0jmUnnoCR01fhrp88hMWn9KOSILMqjUajMufQQNM1LgJ+1q7OTul9efJs27oZDzzwAFr5fThlzSJZtCayUSREkifzDPLLLlXr6Ft9EZqJbokAHrn/12gWD0jBc/3ffBj7dszi0MYZhMoxmbrFIgnEogm0Yuxx2qTCZp0m61XDNgIudIIwIsJqHXBTZ2iUJ+6xH89iYBEzKfWB4zHZBbFDwVKDmQxrYvbGs9k0SpWCEytwsmAOQbKEdGcYi45bjL5Fbdi+8THEawXEU3EBs8RrXnfjp7Fnqq55b7RbCocS+P7n3oALLngJQulhFKa54Q3V9mWcNyb0m2+OSDS3eY9syxfasEf3fefXv/77eRhQUTU+Pm4jbpkqe2dEblxGXDOlNqeGNWvWYH3bEoy/7WuohWtqEXF4JS+S6CKlefyzr5OZdoQbHIdxhMblp5dJRO6dLlwkFuLqmE1e6eE3rgqoUEh1sU/ptEVcxE1+8W3Y+NVbENm4E6GuLJbfchMeeuAJNMINHNy1HXfcdjtefNrJGBjuFEmkmBzCg6FVSCfDKI4fxKcv6EQiYY6J9InavWtSiHMknsWy1evQO7QS5UID44encHj3DMKtjJz0GXmYlgXse7vDlAswVDEBPr/Eg4douVwe7Bh1BAu2TCylo6GYvJeUOpo3NR9QNmNDuwXShKugq3UoHsbgwi4MrBxGOEjh6Z88hqlDo5oyoEjVaiLbHsPQCauAgSy23XMAx5zRi1y4hFYoiliUtaWz0E1nlG7RhJ7kiWwmo7bUX739HTjp1HUY7O3HxN6NOO+01UhlNULc/KF4knLj1uoYWncpCi2qfkJ45rHbUchN4Lrr34MdOw7gwKMB6rPMMmKIJzkegrUr3TzswOJC5zrh1AFNwZCYgCouIpos11rIZGn9a4wrDz4RByFZhPeUG5seZELwJcYgDbQmmihpsfVa1cayhO2ASkVjKNXKRvmkk2PvBE695HTM5HehNXtIffFys4lXXPtJ5Ko0g6dpQ0ssugf/691YfNwZCCIdyE9OIuxYXv9/Nu4LtYDmDvIXiMZz9S1bqAHU3hRH++sfulpjNj2STPiZtSajZritDW99/Zvx4OUfRv9YFWUO9Q0a0qgSU+OLaTLBKaKfYrQwySYfmYvQiQV4E3giakKd5CG2uAVUaSaa+RboQzohtUcWiTSL7ujkfiZcCCGRzKDna+/C/f/0HXRs2o9qGFj/u8/j0c3P4cdf/yZGFgxh7TFDWhCToTZsjS/BWGoY/ZkqTurKoK01g/VdeRndNcNRKW9K5SaaQRYrjj8NhXyAJ+7eiWY5jmSQRTJK07KyIoD/TLwU7+Mk0MWl+joI2f4IkRTRpl6sH0rFQ0pqGA0Kt4jryfY8LAlUkQ7Jr6kH7HqWjteGYpBDrDOMky9ah5n903jqJ3cp6nJywPpzTkPn8Utx/2+eQKsUQd/6djRTVHwRjmiJWcWDktzzvr5+/W4DxUr45Kc+IVLGmtXHY8XKFRgcHMTeHRtw0vJ2tCeJS8RkYkcTOtIQB9ZehUaUHtoFbHnyTrz4nAvR33ssHrh1G0JFNwhOPttpM4j39rFaNJR5RrV5D48ddqbvtBsS4VkHisz+3ARGmRQ4RhXvC1NUlnEkPtAhRL5ijYZkebzn5KdzQ+vQ9JMfKQ/NsvVWNgAwEUE9lsOLXnk8xkafQZ3jQWeKeNkNXxDhwzyom+iORXDHTz6AoZXniAtQIoAXCsReYp7N0sZrjL0HwP9oBx0ln1fsOYqk8UKRmBuVpRS/l8+N4KE32At9+X1XBfkCJVGqpFwqA4TjCbz+DdeidNcmFD/yY9RpoK1ZKnVUgiZqPI3omsHZn0ELiSgjp9ViVGjw3eYG/BJVZBokiVgY9UoVWfZ2XfQNmnWxlXSvnG8sN65O5mTK+nxOZmZ1CaV0WQz998dx719+Coldh+Vn9MiKOFrr+rBquButekH1y2TbSvyu0oMgkkF/OoorhktItKYxsmBYn5uACXW5zAZqzXYsWXkidm+ZwdaHJxEPEmKRifwgIoQNreZnNA0zU/2q3TkN3wqLqcVoy4g8ODik+lcnqrdYEXKcVirsWVSMsvTnGh4Z0kMi+urJCfwvFzEXinjg4SjqdeZGBay+cJmMCh7+7s/R1tWGkbPWItXXiQ2/26nIMnBSL0LtDVTqVZvQ4JhoKSmh2sxxolHRDCRGP1r5DAwMoVgsoVQsI9PZhf+6+WZc97oXY+FQCrGALpxllGsVLDj5GlSDMPYeOIzKxG688rLX4g8/34RosQtTM9OWlgvDOJJteDCK94MHGw8SbsDZHDnhZpFLbTP71myRzecyc+MKvHSjZmy9UOJY0+8hMkx3UOv/0kPM7GR9RFd0VvvGPLzYimPWkRho4awrTsOOZ36DbdsP4C8+/E2Hu9iOeN2lJ+Gjf/s6tC04AdViGZViSZx2yhI1b5FtR41OsbzghV5HGI82GfKFXkdvXMtgW4hHzR2T94Ke457aGvrSe66aG2wtIUsQYMGCBbjqytdg9y8fQuXzv0S4WBYPuchZIZzFE4ZQ5fkblxvS17UaHiKKoYnHaRKn9JLIKf1wqf+UCNqRwnVCBjYJ0NW53KyefM8Tle+p3J4pJ10gkiks/cO/4t4L34n2XFluE5lLlmPy5Da1UHhIFDIj2BJbiH2zUVRTKRzfHsKFg6PoiqYRontEKY96JIUo+UHNLBYvPwObN41j15MVxOnWWGPmEHIjNG3TKhJyKnqCdVtMOmSypJQ5hAJtVG7c4cEhM+d2TB2zPJUd4ZEeYxh6H24a1mVqkRklfq7eTyWSSmN57eZ6yHlABiiVG2WcdsUa/OG2u7F8aAiDJ6/AH371OIJiQkDMglM70cxQUxdIqmhtmADt2YxcHSbGJyQG2Llzp4gqmQytUt2w8loZPZ09+Mb3foBzzjoFs4f34KLzT0BAMghaGFl/NSrNAFt378FLT1+P3c/mMfF0AzFwYqD5dHNyIfvFVrMypbeFLvFFyAzQLdMiQ6wsVRb/3ffxGXG9nlrtaqeMkiFBzAQRsrVNJPRMiMlYKspWkrH1zB0zhnQ6g1yBEcs5PLoh6mwFHvfKxQjFpvDFL34B37rl0SMbNwC+/Ilr8KqLz0couxBT4xPKquZvXIFSDmT9U4L5uUkTDoQ8OuIeDUhpDbjsjbiJ16ITmCI+0NPTjdC//M3lQaVUAZdYR7oNl1x5Ffomm9j0jzcjtYXeUzU0WpYYS/3QMgd+3nKf/un0m0fnkku9NquG3ZieViMOzU+XD0fTRwlaOSKab0kxCul7mSI47ylRvTiPxonr+Tniqxah55sfwtbz3yn0mLDFeHcdnTecIiBmJ3pxqG05ikELhXoCK3szuGgxhxGTwUPheVS+WqEwD400+oaOl3vjY78aBWdV2pxdI6aoZcUSwpl4+2xCEYQaWDXjAY4rpTXr8PCw0nn6RstbqkHXCjOCZy+OAArbLpwLxDRWEr6uDkUfLbzA1CqKtGSJ1ex3mzyR2s8kIrR3pd9UuIizrj4VpYkxbNk0huJuShmt5ZJclkMrxjQ9QDbZgUjcrGjp7HF4bEKLvrszi/EDBzBLhU+oimxbO9raOtRZYLP/jxuewvihcaxYuRLReB0pjcoMsO6Cq9UJHCBIAAAgAElEQVQymZmewmknnIG7/v0pRBspgZoh9toTcYyPT6hdxA3EqMQD1RBiUwlxbXlQjwuSm4ByT4/K8qDXuhC4GTWXlgZlf+zvGwmDmYW8tJwzpt+4mk6hEbCGkZgtEbM4Z41LJls8pjWFTAtnXrMeZ7zkbOybkHjYDuJoDPd8751YftK5CIXimJmeNhFNxAziuUZZNhjZwzJB/3p+BHXdE/fPR9JkI58cDU7Nj8g+TZZE1Q20Y5kT+sxfXhqEolG8/GUXY0FXP7Z88gfIPnEAiLG9URJqR40tdYdawMT/ND7DFrTAJdUtR6RTcdbIRN48b5OFPp35aMjmUmEvPPDjNv2HZZ3X2dY+N3PFEnjrmc3d0FAU3R98ExpL+rHv+s8beMOJ6h1RhG5chkIrid80jkU51g+EGzilK44Ll9MKLySHBdY4HBAtCh5bK23HoqtrBX73H88g3ezQw+Tm8iNQdPKLJGCgiGbUOuN3Xg8JKeoNIkBfX49NDXRRmJvWxlJwIcXQ5JAzDTQzJ0GK5tnL9SMuuPDoDOIXhr/H7A8zmvO9bJxLSDY4QTSBkRd1ITWcxnP/vQNNKoYcQr/otFGEMtMAUmiGqkhEF+PAnho279yp6fW7dm1Dd3saixYtlJa6LUtKJQ/hMA6PHsbuXU+jWi5icjKHgYEBtHdmZLNZyE/jFdf8lVojy1Yci8d+uxWV3TGZqzPzSZEt1uLIy5yMGFiTGnvNi9RscBkPJj5XZmDcyOxZlwp5JNlXdb1e3Sj18zm3iOJ7+mZXnUtkTPU5D1jzFPRjVRtKhXmfaErnN69lR3Xpodkvnxu3GY7hhCuX4ovf+Ta+9u3vuh5zC7FGHU/c/gn0H3uuDO/JWOIr7twcuaY5YcOCjnWXj46e8xFiW7+OeDLPLfOFIq7/mth2kTDGxsYlmeTfOzs7ENp730+DdCaLrR/7LhKPbEfAcQrxGKLsJ7YaKIUDzX5Viurm0BKv4wf2PFOdmvOkSxoxxGkFvi/bbBmpgIQNN6uGIBYXszyC3Ga2E9R0uCKHa2atG6I9r5iPdLZj0Z1fxYOX/TXaxnKgElgT5RIxzFzei4cGT8CziVWoVetEvpCuTuLCkRZOXpxGF3unjiLHeB8JJ9C7aD0ev2MclYNEP81VkadxscjhXdY3thnABKNs4zI6yhSedjq0gG21xCUmMOLBJ14Pa15mJNzAFBkImJE1KRddWUZvZFzRelSCeicwn9u4jv5otkIhtLe1G72QJu41m3JYQA4X3XgB7v7GH/QZJUrnwh86jJ7hHrR1pBTBSRlsNCM4PHEQd999L/bu3YXwzKSM87bt34cgTAM3G6FB293ObAsz41MYXrhIRu2DA0Pyj56amsAp57wSmWQCQ0OL8Pt/30YTSW2uNGcAhSKqH3mdowcP6cASycH1bU27S+F7RAcRa1NGHn7G/OyMwCZ1J3g/2G5sNJFMWDuwWiObyyYYWDZk9Fu2lqjx1s+xBEnSe8zsivje9LYiqNTb06PNG43xWVuGw2fYd0oGQ6tH8PEPvFeHAUe9DA924UMffiO6+46XXJMHC78/6e6RDPfnlE1cVV4PfIR+8T9BJ2c4f9Sk+T/VJlJLMBwSHsHrZ7Yl7fDjb7ouaN2xUYN6a7WyNgwL+UqNIzUomaE3Ygi1SADKhllnJTvbEe7IIDLQhXR/N2Ld7Yj3dAmsaRJYODyB2uPbMPHYs8iQjsaUpUrChiBl45UKKWa/17ntuIgtNJoqHl27m+cTCSPWDKEWbtIJHCt+9yXsuv1BlP/lZ3pPotriWUeB8RdncNeZr8e2mTriLT6YCBqoacpBfnIUo1u2Ij27F6evW45Tl/Tj5DPPxvFLT8bjvxxVRKsVCTqZCwgXlmeqJOOM0uZIyDRQIzUpgo+GFTm4YJgGcwFp0gPvm4EGQq40zZ10zqgza+fw62RMvTljLFUE1nChOeWfO73JeGqoDibSq1Nehx9TXqbzYYQTCSw/rxfP/nE/GhOMygROmug8Lo+Jwqz6uByhOjDYi7vuvN/8nQHs3rMb9cIE+jvasW+sgqo2SgTFUlmeWSesGsHCRUMY6O038If65MIspmfyOO+yq7BwZBjbHx7FxA4rb1hrClGvtnRNqs3CIYwdHtN/6YU8xyHmMvfuIPPMAhltZ2dmnJrK0Gmqd/yMIf6X78FDQUZ8bnCZzdYN0CZdrY0B5YHBTUy9LjcpTfdsdpUNPVOZ4xVunU2cfc2peO97341GuagM6MY3nouVJ52JSKIbs9Mzc4eFNz7nNTbny/H0TNxIl3kg1PxRKKZ0cbFX5aOjP7qRKEfSZJskwetkn533ngc761tluRte8cYgTOJ2bxtiw4PILh5Ez4oliA/0IKDUjNGJ2A0RPBb21SKSDoXNlUuIFmuoT+UskhIFI2gz0I9IbwfC6QRq20ex7X3/itkNWxBiZCKn2QZEauNycr3YRWwhEYBxHj6+leRPoiDKTR7F4q++D5W+Lmy5+iNIShroke0AzWgNtXOX4K6zLkYykcGuXXsw1TmM3Ng4cvkKipNjQKWIanEGqWgYX3n3m3D6iSuw4fdTKB+MolTNIxqwjmqIoSKLnURC/UHR3yJEdFl32onPGoosJ95QooyVkknQBMTQSJ2UT5dS8+ustZjCsfZltO2l/pe0OWY3NTeaIx6VD5ZSMpdicuFx4xAp9TU3nRrIGKpV+VwiCHdWccqlL8J9P7wPcW3cFtqX7kI9xujSoUl3iXgffvGL2xGJBqIVHjp8CDu3P4flxx6LHXsnEGVUk79xSZ/vjJOX46KXX6CevDjfrQAHDh7G/Q8+gnf+7XuwbtUJuO+H29CohUWW4EHH961XWcuaZJGZBaOd3RPLKNQCc7OMtZHmAZK8l8YQmhE6LL02HSBr1TmXCsM/vJuGcQj4d66neCImuirza1Mr2ZA1yva4eZUdaoKCpaCMvk0iJJEAZ71hPV77xrfg6ac3IBEK8Kuffhgr1p1HiY2ki8pEvP0OiSBcz/Ook36UibKBeYPc/yTpQmCVi8BCadyGdoeBzZ6mCQM9o61t2Nvbq4MsVNz8aBAlW6reQLFZRf3gJMoHJ1A8cACNfeOo7h8HihW01YFEyShq/H5uVHoReeYo0UQ9DGkDNSQIhZ4U+j53PZLrj0PjqX3Ycd0/IL9/FNVIC9GggYBEDbGJGGEtFQ3XW9b/dRpcAiSKvuEIlvzb+1BdMoznXvV+pAnkiDUUYUmmGTitSAuVpXFEb3gdJlKduPWJLVgzMoRFmRB+eu8T6FlwHPYf3I/JqSl85f3XYXEb0DuwDA/8ZBtaxThK9QpSkagE9IV83vTBjiEjLnHDVCxWo9oCZI3KTaVIosmAPO2jQpsZidOufuMjYQuG7QsuaAJYQdMDGxYhuGjzhZy0uXygXtbGRc/+rlEnnS9XiykkQas4CuUmcuVJXPjOF+O+7z6MRDylmvxg7RFUgxksXdSD3p42pNo68atfPif8gqNhxsZpdhbg8cefRM/QYkVlCk34+fp7evHRv79RSp9GPauv0VvqmWeekoHex2/6JA7tmsahh+toxlqyzJEEjwPf8pZ1SCpaNwEBN7TfuGrvhUyJxsORm5cAH1+WxlKvTTKLlWjcvKQt8n5KJSN02uSZYvjxz37gnEa5BhpPyvfnUG/+Pg2Uc9MgmQQJT9U8ZANRYqE4ll3Sj/FaEa969RXoSSVxy83vw9IV58mMPed0wb6zwc86f+Nqs7oZODqc5m1cX+ce3bv1I9TtGv9nes2Ny2ucnc3NXXdfX5+yr9Dm5ecHbOVIhkeYnWJ02qW6KQJmim3oHm+yRyy9IZbvzVH87j+gDUI2rx660U8tG8Sx3/kAKody2Pu6j2Ls8G5EeMCQVyYbbsrd/HR2MmysnURieoI1SiSMVT/6LGYSUWy55mNIVmpiO/Fw0Oeg6RiF+OEmKovacOjCfpSDFEIa38ETNYJnn9uCVjSFBWtOxFvf8lY0y3l09XZgz7NFTGwMoU5fI9rHuBSYD51/N9UH38FNfRd7xxYlI65GPc61tawtxAdBAMWnYhQFsC4hH5cnd09Pj5kJcNE5/2iJpVyflWZxdnABhWJOp6zIGCQhubqfMct8p4FimdMRSzjzTevw8F0bER5voRkJMHBSGxBnCkneNr2CiyiVCxJS8M/ymZ6ZwMMPP4zp6SJyRdqj1rFm1XJce81VQCihNLNcsYHRBw4ewMaNTyKIxPHtr38Td/5gE2qzTWTiaYGXMqCnVRCZd26MCwlRfmqdoq7v73O4tu9E8P46je6R7kJ07h4yc+Gztt6mn8hgBxjRaCmaOKZlbjoElWZxgX6Msha5jcQhQoZYpm5Gs+u/xmMhtC1I4ZTXn4Qbr74SSxd248Z3vBEdXcv1zMj8EnCo6Y4WGXmQNI8yjffPf370nNsXR1navFAk9lHdZ1xcg7OzU4jH0+jKtiOZjeOhDbsR2jF8WsDFwyI7iETF9+RN0DR417f0fsg+AglPcnUSf5YEhQa9drxDvktd+MsF3bdCKHTEseTXn0e9Auy+9K8xeviAicrZD9aUPWvUk3qmjciNQWL1QD/W/eJzmNl6CLuv/wLitYrSdvPCptmtsd/VjkED09kQUu86G/UgpgiIUAxVEtejcRy/9hSk27tQD0Kq45YvW4E7b96K+rTV2easT1vXqk1m10gQWr2S8eVsNx1pnAuIG6pSKllaywdaqwosUvrbNO9gno6U4VGXq9qLM3Gdo6GiJ9tjIrAcsUTlkEaf1hnQktT9MGGPmyCvU9oECoVKE7VyE8klUQwtH8LuB3cp/Rs+sQu1cFnti6Y40lZ/hee57BNTqFTLeOLxpzA6ehjFagV/dtnL0dffi3yRQ9PIC45q3vETTzyBZ595Gu/54AfQmx7G5jundEBX8iWNDNXcqGQK+ZzNOubhVGYpxSgqK16boKgxqxK0WNRUNtM0b2hLr4lC26FuYF3UKLbOHI4/M3dYzpPqcREoisfCstvl2iJmIMojPcyc95g8qmWfaxE3FqO6KowgHcZLr3sR/ur6t+Kay0/C6eddgFC8R1MayKbSQeHUVUqx2XP+Xzau750fqV2PpMPzI7A/sOan4irTaPlTt4O8Fs3gKz/bhOem2xDaNHgqoTlBRIlsB0qFgknOPKWRBueudmWNZrpdLmZyROviuYrVMs9Amy0Spot68eTl/ygY7+/C8t98AWP3/hG7bviUhOPynvDDmIhcq94Io0p0dvkCnHvLv2L/rQ+h+PF/l5skHwQfojG0WmjwwYQ5cc82SzEWIPb3F6LElhRqKAchdLZ1Y/W6U6SxTCTbtFAr1Tz6+hbh3u8fkvsEGUnarLG4alAeUlxk0sSSxVUlFdQWAaMDCRMiELgDTO0Od9AZsmuTzRmpIhGjdJL4bv5E5NUSfY45uR0JCXa7VHuFjcBgabeBLKI8ztu4/s/8mVKtiaCWwN7pvXjVuy7DAzffJx/g933hvWhGK1h3/Hq85JyX4OSTT9Z8XSL3/sXowc1pw78bGlxGOI9Dy1PpNswWZlDO0ySgomvJFwt43TWvxUO37kYwDkSSEURaURwYPYS2bFYHmEdguVa4cf3MIhkpcGJfqaxaX1lZk1pic7rgywM//C8jJn+n7oNvB2p2kaXUtnkt+2HGxAjY0c5h6GYazx6hGG0uvfZsNNswFvG1sUI1RIMkamHgnL9Yjb+4/m34zHsvxaKVZ6IepDA9NeUAR9u4foC6aLn/y8Y9OgL7++5/99Eb2m9cHlgqMXj9AL720434Y24QEwViDTWENnSvD7hYSMNTTUKrlFodcaF2lk54l3XeALoh8KbJPqMVCBVVGu34lJ5v6rWJfuSmasBICIX1S7Hi5n/Aczd+Hodu+TXyTdZIDeRCdfSduRb1YwZQ6+7A488+g4995gvY/a1fIvjOb1AVS8Z8/MyTwOSE9Le1ifI6JTR4KvyBl6EQM08rpn46rYMYCvkiDk1MIZuK4uVXvgm18Qx2PEI9px1EPIHN59ec9326It6sSBhmcs62j48MjOp+M9shZK6MjIRcpNygpBiydh0c7AOtVkj+kEWN7HCNtxximeKmETACcWAZWxeK6AS6KN+LeajyiIsgf54G5PVGAuNTo7jk7efgnlseIrUNn/n+J1Co0eOZEc0irmcrEcEmJ3jJ0iVYuHARli9bhsULF6BaLQlA7O/tRyrbrnp/cuIQanXWcFAv94Tlp+Cem59BiCNA3QAvZmjjY5OqBz2SzoyIf9dBzpTWfXylxUqpbRN6Cx4PXGktsiSRQZo1ctm+4cNXhBb32owN+bM8ZEkHnNMtN41ooXZT3AlmJK90UdNlhp5Qw94+sZZWDDj9qlX47V0/x0vWZDCw7Cz16GlGJyKEk/ERSfb8ZIa8uZcfseMMAvzX5+t0j96oL7Rx+TZJSr8QxbPbD+PLv9qHg6UU8jVzRVHb8I+dJwRMdRX2nfu+indnpanUSu/uepmIIJPNGlDA044pjecoz/NAtjEgNj6YPTW9PxUiyRjav3gjMievw8NnvgWPlHZiwaWnIL16BPlwHcVcXS4Df/6612Pff9yN2uf+U35INqjKUqRQJCTnQHF3xY6x/IDyLk4wr73ueNSWdYKGKV6Zw0lqXALcSATCzv+za3H3Tw8gyMclVayWbVwJf4f5TBs1T3B8rarygWkw02PtAvV0G+q/8iESoCIyLKoneboBLWksarK9RNUKwaVyqaJoEwoZ19lHEppwC+yS2VxNhAfxo5kFxNkHroi6d2Riu/GfmU6VK1Xkck1Um02cdtVabNu0HcXDOdz6wI+Rr+VQKZeM3FAqKWJUa7w2ShkbqDWcOL7JSGtYBqmHf3nD27Dm+HW4+977VAotPfYY/e41x6/GjgcmUdlPIs6RXj5XSblECx8TSIgHnEza3x1ZXlMYnTCeRAulwSIYmK2PbWKTryl1pl0OBRoaMm1kH2mUE2wT2SHEDIxAIidDSPDh3Vy43pzxAIejKdWUHJCoNYOSbXrNIpYIhusqitXnD6N9aQaNyWfQ1rcMM7PUWFuGoo2rWUMmO7RQcaTv4109ZBTgkGGTeBpngRf4pxDmuU3OSEvmYTyKJ3fN4gu37sXBSgwtMtmcvluQ8PaFZwWMND6q+NrBi9z5ht7T2Gh3JiDgQiUB2tP0vCujTjFnJcn3ogiBvFoxkfhQIiGMpcM47tF/x6Z//B5a/U3kO6pItqLIizAODCxchf7+lRg97+0oRo1iGW858MrdFCmSeFNIkVTeaF5SzWYY+XOHUDttRHVdXIO9OHzZmvH8fyiUwDkXvwl33rwPKQTIF4l90EW/rtYF6zRuRn9PRHiI2Exg1V8y8HKDoV3tleXh1zCvLhFTGk2UikWBeb29PYoYrOt40wnvc96Q0mKJ1MMInCkY0de2bHqu9mUNyujMdJuR0JcgfjI8a+RymbOKmogk4lh85iDqrQp2PrkFO2Y2YqY8Nec6yefC66rUawJcKGzIFUwEoXSTwFzdOgepWBRtnV3YuWePWKvMXLhhHnv8Gdx/8xNIVJJoeHsescZ4qIZxaPSwFrgGeCkVNbYcRRfqx8aYFpcRi9hnkRjdWeYSwPOkHgM2LYVmfcznpvqVLUNHVmHtx03d092tDMhHRf4uvg8R7UJxRlGaNa7MDqoVYRlkonET8XdywwUtHrpJBL0VvPQNZ6M8sQHRZI8GmvGpqU3lNq7cT53BocwU3ctvXPVyj+xEy1r9YID5fV+vTXcBT+HRIcy/uHsnbn4iQEnG+mSlMYjYgAAZL2wbeXHg3eOPuOVTQGH8WHvNS0c1IdMkYr4RLsBhvumzZqtyFoy1dhjFuAnsQ4WM/H3Tteh62ZnYeONNKFzcp5lFjN5M+84470o89fpPILNv3JRGfGj6PHZqeU2vlTimnOAG4FZmWlw8phOhN58oK1JuFt5QZhNEYnlyvejsl6JcGMT2PxTN/5h80ybrIjvVuFisbLAHZEJzoKOjXRuP9SgXjBBOhwXIM+lIJiu6H/9dM1c5ST6bUdpGDrT3VmK0tihqtbOJEoBEzJm/sw/sFwWBnWZFogePQPvnUy5xQTY1d7htcRrDJw/juTufRiW7Xy6PRO+pKOLi5rUVCXhUqjqomLlYthVgZnpWYBrTwzotgFjr03OMNXCliVe97rV4yxvejg237tF9YMuDP2eZSRy52YIimqmOSDYxm12+uEnpq81SRBvQtXh4nxhd5C3teq8G2BkPXNarLlJZL5jP1MQwjMw017Nsy4wX5jJAx0BjqcFnxfKEG5iqI6HDySPOjmxTMbKr5xxUcfHfnI1qbidCkTjGxsYUxeNzRg4hOVZKoupagnMbd95UvheqYedHWz9EfW7Xa5hACPFwGN+77Snc9kwUJXCOFdc3cRG2FNxUBQavrSNn6dbyhPSsD90cpgNucpolzs4lj7rGpM1Z8SkB0zVK9bzJHL/XR27eXJmTs8XkjOi44Gb6M1h255fx5Gs+htClAyjEq6iXa4hnO7B2/YXYd8nfafFYP4yxVMN7TT/nUi6lzrx9Gi1CtQijRhOz/XGk30V+KQ8Ja5moppRWs4WXvuqNePiX46iNRWWA3ar7mTVO9+lGPnpvZAm7nY2qiFBCZ+0UjbvBZb5u44LgK5+flSKFBwY/G+1R6FAoET1PcEZS0hmDBhJxo8vxACToVasWHUHAeGWemM90sVIqggB0nGCca6fUG4xGtpFqyQrOuvoMPPZfD6PRvR+hSF2icrW2NPLTDiOPX9Dojv9GJL3WYFupLHF9IV9GKpm2A7FZx8x0Hh/9zKex94kyigfokUUFFrMB6/tycRFDkClIKIR8IW/SPi1u1pwcVGZaaoJ/Att0CDclJ/REFAMIY2JK8XkzQs6NJ5GayGYpMVK3yd6HaqmW2H5ztq1UshWZ4em3S3lktrgGRumQndNEM7BwwqOVNASeTvzzY5HoqKGSm7H+c5j4gqXJfLFuFxg5X1MrEc6RfXIk4DqXEx8C5xE25iv8WFLSNfPff70Bv34mjCJsrcTTZNORLWYZpR8eF9rYc3LA09AMoW0atxA3OeVruzqswT4A00XaWTINlOxOobuFbJL2KO6CONfU1QDeBI4nlOxbHMLXjAJDt34K9VAE93zpn5Bbau917LK16GyNYPz6T6AZNXI6HfbpRuBPLA9iPH/jUulBW506RqNVjHz6KiGkRCzllhCn1I0E+G6ccM6rcdf3n0a4FEFZg7isxmIbQ3QyotsyzQtEVGA08MwZ/hvfkwudJzSjH69JIojACAdMq9mOYOQiP1nc23QCcQIsLomSGUA0JtCKKCgpkh2dBnoFjaqzuXFSSXGlWQ5w1CZnzNuEO3+qRyIJ1BsRFMoVVCJlnH/92bjn+3cjMjCGZst41Hx/z77hVEU9Zc5oKpbVj6a/FFF7L7tT31JZQFP0R0ocb3j33+H+bz+HUDMhk3v2Ejgnie/L665UicQbWMfsoVwqI+nQdT4rblzrf8esNUPVUlsG5ZpxwnkPueG5oNva2sWA8tRTH42pIGrvaDO+tiR7jpghpxRuSOvTckPzuUh258zluL6Zdstt05Vclm14bjTvdxQDZ2Sx7JQFGN21RQe06vK4Hch8sa999MbVWpy3Keei8FEDwPxmt5T3iKVxKBTDfRt24yt3TKPcjCOIJBFTOUXTQmarRGts6IAyjyc7Tgj4ZppNE2f9YD001miG+pl3lOeYdrV3GE3Mp8H+w1Ijqj4oVTd2sZ4RI6GAH1btEDf++8xZK7HiK3+Pu6+4EUuvO0tCx2imE7nxMCbe83lw5LIALtYMtGadP/xXd8YAGlvUNiqF59JMpIWRz74GuSb1oLSBsUHJBHrWvvjlKE6lsfn3OQdImSRLvGOe2hHblKQ5cm4Q74e1dBghOZg6JldFLgJ+tpT4sG6siJvVyo3O+iuRsJaHShlXm8TiVtsxE/HaXKavRHipWJLXstg/bqj2PMCPN7ZWLStdZtS39w6bfVCLA5lt0PXZf/ki/P4/7kHQNqrIrFlznE3sRlkq13QvZlpGBpkHqBCwcUbiPGBKhSLOvOQyFEaTGHsir5q3QsM0URxJj6yq1ODGK+TN5ZKbiuQNuqIoGsq5xMAskUkCAmt2MDPSsW8tRZUiY0htHbqtGLBjBgV8ETnmNbJONiMCo5YqC3LtNJ/t6WASVdM2LJ+HodUWea1OBcLRiLILcYJCYWSHozjpVauxZ9vGudrUYwsqoZy5ok3Pc/fS9+vm7qwLe0fVtM9Ll2WPQ8JTA+OFMt7/9WcwjTY0YmnZvsaTaStnahzknVLGJC44p2Q81XWiM0Q3obv6Zx0dRn9zhm1EgxkxbWK32/FuQfkPwtOUp6IMy3kCayMwzXKsK9/2IJWP/rlM26IxDD/0Zez53I8w/qP/Rq1Vw8hrX4bCypWY/dBXbFzHESbY8yKubrxQYEvNvCkbb2YhEmDBh16J8SS9mDlBwMjvTCXPufw63HXzZgTTxkGm7pSfm6AUr52pNFMjfj91yjwRGAUZOVWXiLFF83i2j5pIa7KCcZe5CZi+8cAiwkzrVxMb2CEoml7UDjQtGNIDqUHVbCACfexvhpFgy0N1HdNJ+zPbavx3Rnv2q9lOESOI1y7taBLleoB6pYYX33g6fvuT2xFvnxQophaPi/TKkhzZRC09j37O+R3bBvYHN593pqcPp5/zMjz2090ojfMwS2rDMjctFug6QbUUyRpGCzWBe0g4yMThMRC447rm16391ZKUL58v6B5ZKm12M6xV+Tv5M1QCMRvgvWPKOtA/oFRZ6bHsd6lAMvDR9RVMyOEGirFNVMznRBflIVcu0zzO+uG85zyQxZVWORZGPEWqaAiteBHnv/VM7N35lK7DJKVO/0uket7oy/llpGM8Wp463+rC39v/8XWKM0KoBjV86N/uw9ZiP0LRhCyBSBhiek5ar9cQM4Mayi8AACAASURBVHD4/n7o8bbj3dawMYEecu8d6AOn2NFipCWWiKUTNr3MwJP5LA/Pu+SHZiriN7hpR63Z7Qd8MdqwtmLU7vmPD6KeTmP3pe9CuVZE6sozkDjxJBz84JcYQp8XZeenygIH3M2xtMXqRG6uYqiF2DUnAauHEYmF0ag1JIfqX3wshpedgSd+fACVotVdOmxicbUU+F9+RhqU8XSjAIK1kjX8WYvGEecM4ahNQVdLQYivqYh4f7gQWA8z/ybwwtm1mjQrX2PycMNSCvH3UnjPeyiuc5P6XLaEmggHpmG1iGoRhx+CRAmZYmtUhqWkXLg8kCKRpAzDOe7mhNevxR2/vAPDi8M4dOggkhzWrXLAMhih2O6/RsQ3FFbAm1hJtBgy2ilbOC+5/Br88ZcbkKkM4sCBQ2g1w2hv78DefYY4c/FyNhDbJpp84eieau3EEyLaGE/btMncJnK6cACWrF8jvNcFpBJsz9nmdbOrVfszI1HpIVDpyNgSUj0ZIFLCFpyxvxu0RrklLXA9+433T6YG6qNz/ZgjBwk/as0RJ6HzZrSC8647DQf2PWMjXnTY2cYV8eN5UfVIXfv/eePyXYMWfnH/JvzwwQaq4QSiqR5UmUlyJAoZhRHXVmU22QwELioDfaxjrVJlnbIOWPC6UD5cwuWkM1LELP4ua0K3YTwyxp8X7d59nYIFRh72Dr1PkC1A9z38PhEammicuwpL/u0juP/E1yA8PYP0Jacifcm52P6OTyFBL2JWdPOr+KNSETvdDF22YhySHx5a2YYlbz5P/s+ZNDWsJZxz+TV4/M5DKOyIiNHj60RNkBdgI4K247Ia+ql6goAK5XrqmyaRlIuE/TsF1lwwMioLM12kqZqRBIRiFktO0sfNwe9rU8bBk7PWrGGQ/Vqi8qRxOiYQf5cxpgi6HfldHVk7OOXCILsX6wmrhaLISxQ6jBUvX4oHHn8M0ehhbRIt+LR5J/u02DOUGHXmUNu6SRB5bcl4Gs2ghjMuvgxTO8vIbyG63kJxhuBVXiwpjprMF8qoVQmaMOMwcYGuwx0MJP9zo9EZhP1gblBD43nomEujPzQUTWS1aoZwJflzWUTm/3VfWTK5mUMei2C05+EkVRVxAL2HqYy4BvnyrC2NQdGAbluLyniSJlAnZkGhCbW/p752Ncan96NSG0cmQ8TbXprV67IXre0/6Xrxv6fKvE/8/X/9z/dgMjKCZrwDkWQbYikzDPC8eR0YPBQ5z6vsNOKPd/iIy2fmhNw6fY1Lyovv6+5BoViw2oSppXcnEDrqDMtdW0ZjMmUGzlMsKtXR3CnvLt4saQI0edGpOIbv/Fds+dx3Ubz5NjRWLkD7e6/F1jd/CMkghBjra3kWz+uXebraUTWv5ztXwsD+jhqOed8VCBJhJIMoIp1dOPn0V+DJ2yaRHy2iWm0iN5szBNNZXwpwopF7vaE2BFsE8xk87GfrnrA/rAFeBHNo5Ba3dNctBuMTOyvSRl1ZC9s+BFvk1FGyOpAiek5akPqFcj5FWRN80J2SiziRosVOzSRt/JqrRTV9SYveAT5kXcFqxkUvGcFMq4idW+7X93PR0ZXCz/eZnx7z+0WcbzblgMHPxgxgejaHk847D6F6Gvv/MIFIPSHTuVYthG3bdittbYU4gnQXopGEEHxrCxGoi9mfmeaqN0y9ctLRLW0DMt0XAUL6VcMMZLimdLklVNk2vVFRBeD5WtlpWg1INEsfIueWNFgLju8ld01xvK1lqM3A9l7NLHI8QhuX8ZuNFCEQ19HWg0Uv7kX7ghRmcns1cdIfEqZimseWcp9Fh59b38+PyPbF+dkp/+4Pt3/+3u/w0P5O1OMdCGe6EEtl5iZ88B1Z2xPxVgChgUOFf28h9Ejb6sDXUX7jGo/TtTvicaGfczYf9L2RiMAr+e1jegIGHwSlbGYcHAicmGs/zAOoGEWJTIrc/433IGhPYsuV78Z0q4Ghb30Qm1/3fqTnNi51u4xiBkZoRIpP1d1dkvLPAQTVoIWpZB0LPvpq1Dl1oQJc8qa34rHf70NuWwSVnOmCebLu3LVThT+nnIvW6HymvDO9IZRUBxlARy4uox2vV6AK7T7TSUOsUwkdxroHHIfpwA5mLGQv8exhROSIjwUjI4rKjIZKT1kvp5lq07mBdTEPPJYTbIdERCAgiOFVWWzHqD+udkkY8XQalQp7vTUMnDSEjmP68Mh9P7FIQ9Sb7RWX9YjcMEdpZWpL8zue8lb/cqEsWbUG/YvW4sDt21GpxFDImWEdSRbbtuxCe0eHShOiypOTMwIAdUjI8tV6+Hz+smGlY4WqbE9RJJLvNhR7Ww4f4PuzfGCqPDw0JE41gSebD2TPXGmrR9ndIC0Dy1ivRtDRYS0i9qNVwpDdRkxBLUT7/VxG1YoRghTN5VkFHTSck8T+P4arOOeqc7Bj15M24REUY3BihVbakbxv3sb1KPH8+bj+G5+/ce2zTE7n8defvRulbC+iySHEO3oQTqTkq+XZWsQseD28JyySWDaICPpY+1pRoYSMuk3ATcpThjeSi4kDovUglJPbtxmiduSliepO4cHL8ubbjFKsaZliqLZxvUfJ+Pyg31ecjp4Pvhlbz34rytN5xL/0Djx04ycxVA+QDMJymHy+K8SR3+3TPP9J9LCCAGORBvrf83IUExFc+sYbsWdzGeV9wPjeaZRmK4riTDX52fI5yt2sXzjf8Iv9OuPb1sQlNufAqA4RXn+jWlebhwuMt49kACO/N5Ei4YLvx1kvmixvaHKj2kBnZ7tmACnFdQtSelJuQIrtOTLDeQlzCh+7SBwh4iWbirp8RhRjiBLJGpqzY81Ct2tJB5acuxz33v4ztLdnMDY+qgXPQ0GIrwO1rN6k+39R94F1KOvyxWuPx4LFq7Htrl2IluOoV62VNDtDA3Nayc6qFqQgpFLiPNy8XE7URZiHgTDWx2XH49a72kQlJFPcyA6s0wRHZiFFHXgExej04QeS0xHD/L8ccUezhoydxmyF7SYjuqS12AlAGYWXkk6T+lk5ZWNMxCngoPZy3oz2SfaAlYTm11xGOJpANZHDy996MXbu24QIsQcX/US6cIezJknOYz/N7YZ5GamPrnPMKR7dQQQ1FPH+z96CHaXFaKQ7kWrrRiKTpZWh8ebFt7Y51fy83LBSvIt33kLo0bY1AReAPoAmk5nxFT8db4D6qM7sjQuGkUX1kRM4z31YZ6XJn+F8VR8RWf36ekfpgbtQcoz5+/igC11JLL//G/jjyW9BtJxD+IPX4OEf/QLdG3chQ1mRU8b4lMPD/fNTEJ+O8waRZjlD5PDqM3HBh/8WhcMRjG2tojLZwNRYDqV8WVRJ/n5DM9lTY9O+qEXNjapF5IyxCckTxWUNZKQLDgbjTB2SPuhRZaATWxncAOIic8GyHUGgq16FbFZLrHfTKBbzyGTpF30kjWMPkveG70WKKP/Mz9Pf34NKuYAoxeHsSTtpmmHJHnCiEiYudlS2pxvVSBVrL1+Lu371X2gFRW1wwzCIskfmNq5q2WTWMopwBFXW4/1DOP3sl2HTHc8iXWhHhZMWNfeX0+Zz+r6JiRkd7FR9FQrcPBmMTdA10iOwbuCb0n5D7bmB1FJEQ77RJPHMIa+thq6V6DyRaNXicqkwxp0FFjusxQtw3lwUshcLeSxZskQOHbn8rNJrk05yE9YklhH45gCtufQcRkll1pRMpw055gFCgCybQTKdwLpXrEQtWUJuclxRzrO45rfT5kfU+evyhTa0slRRJFvYO1HEez/3e+RTvYi0DyLe3ql7yhGyxEq4z3h4kdg0V5p6A0K2g7Rx5/UhFcHCIWRSWecAAelpmRtKl8qr89P0XJTWLRU5w/yAaChmG5eGcZY2zQey3BGoTaCaJhxC/+PfxrPv+ypCv38Q1QtPRLBgEDs//210BMa+YVrpU/T5ULscMlzNoNRHtUqA0fY0rnz4R5gd48jIJqpTZRTzDVQKNREt1CYi4lksoFY1hJu12dT0jOor1U6OTEHqHxegro3v3wo0c4c3lRan/ABsu5ClxZ9tb8/KwzebSqPM6X01MxqjQKEldhI5zDVkM6aCUZSNmhOEDkeqfep1ETJo2VKv0nM4g0hg/VF7mWeT6JMNglQsTyJo6+1BEAuw6IIleOD3t6NQ2Kvszpz3HVVQLRhLr8jt5ufN53JoBlG89MqrsfvRPQgOhjXcKyAWI+8t/r4wxsYPC9hjxC2WCxJ412stkNQhOicJDorkloILMkuQfEJDd0YOpsI1lUk84HhPNc5FKbbp0KSskh1QXFHUDhbbuEqXiTxLFM9B3swSOJmPkZTCBJI76PJovWndI9fnV8bnhpyTK82+uRhbLtXUNQZN9A72IhXN4GB4B172hguxY8dmtBzpQp/BaafnJZxzSL3/2p/auBHSGMMVvOPDP8b+6hCa9NNuX8j+lAbhRTkyJWjo+UsUYnwoHboq4R3fPPTH7vU2rc/3TENAxk2Q583wqiBvVmBpsOtpsYaRhzKRX9azCVQd2VunrzyUjzT2+TVvS6NI7m1IEKDntn/C7L5RTNzwj5g5pgMj734z7r/qnWgTTzo8x31W9J6nyODpJ80sca5mCJF4EqUVwzjz11/FzLZZjG2rojhdQatCTjLmVEBs4NuDYl1IrS3TVqKGxtFmCspNw542U2qe7qxPeRdZs1k5HUYg72SysxpAqIae3m7r04aZ7jRRnM2jUa3pfYylY4boXNyVUh4dnR2OWM8WEAEu1q0G5hABZcRhFGcqVy1NC+Biaklmm998rMslzaRRWob0wRgGTxnC/smD2L3lXsR4T0oF0fz0DIRZmFhE7k9BIMLDqRdcgsl9VcxunEWrGUWjbtkXgSd+D+8Jx2hOTZLOmEalYdI5sqyYqXhnR16bZ+MxSjEFZ9sm7GprRdGgrpqfhndsLdFjir+D2YznePv2ju/zsg7394UKNQKWTCWJzAqoi1prrZgnSYTtS5YxBMmsDWb9X6uVNamwRc6xMayYXbFXnMok0dPXp2wzlIwhtSyEodX92P3cs3P7lHdlPt1RmZ+TnM7fzD4jnL+ZqRLPlRt404duRS3eA3QNIdnVg1DELHk1b5qqrXIVFWpxnTrPPMiNjCRA74mudQFbPV5/amSAiJBQf8IJineWH1IJemDDzWxlOpJmisOer+PB+hPHD13yOb5aTc7RXmCJJHlNRD/yJvS84hxsPfU6zCYaiH36emy89kNoZ/3BZhPbDO4OzHfNI9fYUENu8Dj63/QqLP/oDRj940HMHGihNhMgny+JylatmBsDwThGByMNkAVNdJgLs67emYjqqseddIw31AEDAnpkpm10vHTMFod6oFHjMGeyaU2J54FWzOWRcgQNtUGcn5babBznQXJHMinU2ZBGigxicswgiKWSLmILktTPUiWPVMKQZ1uMRkLhwoln0sj29yGZaUMuMYv+lSPY8OCdKBbH0Qz53nDY+pVCV9kXjqKrqw+9CxdjyYqTsfv2XWiWIqg2WC4YEBONxJUm+tJm755RFIs1AWIqNajGd3Wn6WTtsOZPa+qiy6zI4ZKsjiUH6+NqUbUpD1HyibWhdIBSxGLiDF8CMZVmr5UgV1+fs/LhweOnHaCltptlFWzVmeWrMees9UPChge4uI6Z+VCEQracX/8dnW3ydeYG6h4YQD40gzXnL8Xk7CgK+cIc3/7/tkGP/rf5GSIPi4/+8y+x8XAK9WQPIv1LkcykEAlbf5sBgPpgkZ44MJ3llLMx9k4hyoofyq4ShMyaw99Unpysz+RqSEcEWY2YKsdL/GxhM4Pmmc3hTil9wdtk2oNjjLf+rU9plULzEHCT+PRQww1UXnseFr7rWmw++TpUQhXkPvQa7P7YN9Cey6MrnJS21r/mQBqCBOoXEqKOY/1Nf4vsay/B3sf3ojya4GhTFKermnvKVJAkAfZR9dlbgU1g1xhMmyJYoZdVJGY6Wk0WbJlxma7bXAVlqeMWgozO6GZYMmolPaVYLDdaDSTTUd2PGGvuitVpOvwcOV2gX5MAldH9eAncHOSB9/Z029eUHpqti6w6xVclH7hoKiHH8GKKzjIm3dmOZFc3IskUplqTWH/Zi3HPz25FMxhFHeYVrc3EfrUDClMZaqtDuOBVV+K5329FZDYjsnyrboohEVuoruKCcnYt+/eNoVZpIXC8YJYUHELNtJb9XRJY2BbiRbOG5DPnPeW0Pt4n8pmjHGdDQbyTQpoai5pgI2NISJBg5DYLVqbevF4OaWPrTAIQaZ15z00QQw6zhAt0Z9H9s/6nJ7wwhbbpBWZFxI3MDS4mnzNnZ4eAJ0b/YD8yvR3ItrdjOnQIa89dhmc3bTK85ihgdn5Enb9Jj3z9SHmTL5bxtg//GuVIFxrt3Yhr4yYRallbj59NGAvLDreRVWaaBGpOlRb6Q/a4INwMxHAhsVtjDtwbWI/NHDD8KardzsqFUdgJ23lj2K8VgVxjJU1+NHcRrhnvEWBGT5uT6njGYaD4kuNwzD++BxvOeBsirQam3/NK7PjBr5B+bqeIGElK4o8iYjDZI8OnFo7good/jOnuXow9th+NQ6y/6qiWKJCvKYKZyDqEsbEJRa9MOotcPj/3wLiwGFIqdSpSDBDwNa2RFdiftHTQj4vkwZRxSKoiIiN5g86FIRQqeWRSSU0baDW4cAsiVGh4meprHoYG8vFwjEu5VENXV4csVxhdpL7yWYbIB25iBA3Q6JkrMQhTRANguob65bEc72hDvlnB6kvXY+NtT2K29hRKTdO+MrJwceZzeRNJhBN48aWXYXpvE9UdVQTNxBwrjNnXxMQEUumskUTC5B/PYuzwLGZmiA6b+6OymCjdUdiSMqSejDMePJRCclPQ7jYSbpj3kxsKRyIE570QFGP7i71vWcs6yx4Oqg61YqiRvNHeISdPKqlIE7RgYmUSnxXpq+0d7Sa0JzPKbQCapPMmcrPz655oowO71ZS5O1Vb/LuZEpSwZOlSSnWQ6uhCRz9/bx1d6yJIdWawc9s2M2dwr/nkIGPwuTrd1aN8fja0PYZGqIgf3vIAfnrfNFqJbqB/EVLd/WrFeYop12mZg+LqbJkRvTVWm2+1WXkUIHR/emVAhDTLiMkERpvP0dJc7UtChbXx3UtpGsGKQBFCFDU5CtjPqz/riezzkGRFXg/Pe8E9iRocYbl8GMM//gSeeek7kZ7OI3fNOXh28yZEf/MQkty41CTOO+l4AfT7zQ8P4OX3fg+VYgj7Nk6iORtFpWhuG6V8UXUaWU2cK0qQibYoBw4cUF0Vo4Y0n3N0RAOomkEIuTxTKBNu8/uJ9Eqe6MoA7h9S74g2p2nQzUhCgCkW0UR2kQUoJ1R0toOPQAgb/7EwXS+Y1vMmEtU1twdyFbt7ekVW4Mb21EDWfOLSSs3N1LAJpZxBzTjBXIAuemZ7OpFqzyLd04uZWhHHvXw1Nv12B3YfvgfhjPVVjW5qjDA+i1K+hD+77u147padCNdZY7PGZAlhdZw43rwCN1FgapKSvxomxvOIOg8ylVQsr9wi05S5OMdC5uSzxfvOdg9TwGQyjmicQ62LaO+JINsRR7wjBLb+YwkbyOXBrWqJnOwQ8lNljO8sIKjE0ZHtEoLPZ8MsTx5ebl3E4sYnlxJKHHlnbyNKI0UiVuMqnachBANGMT+nhOOa4ubPtmUR5yjObArJ9iw62zqwv7ATJ1+4FvtG96FW4oxae70Qq0+HrV+rag2xjRpDNWjgmnd+C7nwIKJdi5AYWoBwOmsB0GU0co7kYcyfbzAzkPRBb2dSTPtz6IHscUFc7o5E6szIWoOU1OwmeZ6nnvOfFVDBm2FvQhTZ80WYemiPUq6mVMcTrT04xVPyyER6r93VCcULWzSIgdv/BU9e8T50Pr0XB4fbUb7qRdj7ia+jB3EkXQtANiNKm0KIrT4WZ932PUwcmsL45gaCfBPl2QIKlQC1EoEd1l8t0TW5mJg+8b/9/f3Yv3+/wCC2BKjh9QcNPYRmczZwWYR1Z9BNhNTYYIZa8qWay5P9pQnmQC/WYmHQrpbkCD4QuTbWyygUaPNZ0MZRKhgmAk35Wgr93YP6XUoJo9bP5f3V/ReHmMWujafsaqerZkk6WRrmqSInMb+nC+muNqS6ejFZnMGqy1Zj6x2j2Hv4IbSSs4rMSiFpuCePYfkE4pVvvAEbfrgD0RBrSBJcmMITLDGmGK1x1Gar1zE6SmF5HHkSMlxfWCm02xCGYVgLkJuQBxZ/doajRUJVdPSEcPJpK1FJHha6ykgd1JnCsuZnVmStOLskO5RIl6zWSggV4sjtD9CcjSPCodk6LA2TMRqkyfr4u3mdbKsxS+Kf5UDikHhGZ6EWnK5YKQv152Zgq4n3PNOWVV86mY0h0zOIbNaR/kca6Fnajp2bDagSc3deFjg/w5y/cWkvzOf0wB934rPffhiNRA/ifcuRHBxBjPOZKXap1hR1fe+WtbtIR9q4NvpGskQCoXzuj7avkVmcB0Y09pD/88Zc3MBC4MypkOCTX9BJkbINJZ1Le90i8uGdC1hfcj1Hf1IJn3Xu7GFuhs4khv7wTTz7l19A4vd/RK09jpn3X46n3vFxLAyldcqKG8rFhhbazj8DZ9z8BRx8egwz2zn2gkSHGiqFskgObF2w1tKUPFqQcpaNc+XgZzAksSUHP8q0eFp7WRcjhTX46WVsKhf2CT0QRP6sjdZk7WtqE25GpuIkSgTNKtCsYHziIA6P7UGrSVqj8Y45aEwAl0tvfUrOKMrabu2q1Wgj9Y0T72KMTsyE3Oneagjt5M8kOduoMEOSI6wCJEDZj0gmgUxnP6ZLU1j1yrV47rY9KNXHsO3QHxRJGPHiSeqAC+aK2DaIc/7s1dj0o902uM1EgIhFDeXkM5+cnhJnmKf9nl0HEQRR1fUc68Lv8SojXwpR2ULQJxRuoZDLo9IoAdESzrp0MULxCkplTp8iDdR5kSkS2ybTjB+3YjSF0bVodM81qK1FwB6TW8qY3E2ZZVqZUyxpkxRMKBHRKBJbm6wbmyIwZNNJJ6yvzE1SUKrfqAgk0+cPWujs7taG5AbOdLQj2dmGTCqB8doMjjt7IZ579hmNnqFAgPZItomPjI19XmboWqHEC97+ke9hX6EDQXYAyZ5FSPQPWztP9jQ2zbBJphRH68kS2Ea3KrJz/zmaqOZXsR1kIdhefuMaN9hFUaalHIdAXqy4x4Ta06hpSp27za6O9Tm+P32YJvq2j1hNDlnVUe+yb6J6QTqKkYe/i22fuxn43h1oRAIU3nkp7rvpC1gUTyJFCy1ukgBof+mZOONHn8eWJ/ZgZnMIyHMKm03N0wgWWo06ckc6lTErFkYFprqMUAJ7rN/IBzo9M6u0j0R9LhS5J4gDTEvVrDY9oTZTvxiSy0WnVlmIJQIwPT0htLRWmcGh0e2oVui95LW6jkTChe7wAuPz2n2XKknjWCxapBMJ9HR0YXhgELFIco622Nne7iRm9pQ4lDpUr6LJD9BsoWfBEOIEOtJZlFHGsouPx7Zf7UEQrmDz4TvcLFoqT0Jq+fF6lq04ESPL1uPZn+zQac5+bCQes7k/DsvgY+JG172aLiJoRjE9My0JGg8btnr881YrTBGdhJUois0pLF2TwfAxMc3z5UahAGV2pqCNSnosQTmLKMYFsJ1gA+CYYfH9GX0kDuB8JqWTAcLVAPs2ziJR7UciltIJyufFSMu0XVkUsQoZHJCBZsoqK/NsM7PmJ/PMwDSzE+7o7tThlU6l0N7TrZSZh108nUF8pIH24Qx2bNtCtficc+XcBvKbeN4XeKgWKlW89m/+E610F0Idi9A2tBiRjB3CygxbTdkJMftgYOLn8BvX6lsCwQZe6faQq+zLUAJGXLB82QLz99CRLxh9CdK4ERGs0bRx/ffN5w97JZDoeTbvVfWFK+C5AX1KxHQp2p5G3wPfxN5v/BzVL94ix4vZl6/HQw/ei+HRKYFT5PDGertx0dO3Ye+zh3DgAQ6RLsn9QRPxOHCMzm9y5LNeq6HFjIaOteX+K3MA+hvXaihQuscSAUynTaxsfWabycpFxZRKG52nvqNqEgCxYV4VFArTGJvcjlxuDNFoSbUsDztzEfRAHVHmhA4Wk8+ZWJ7fx9Tf92WZsnGLE7Q5cc16dLZ3akGypJnjG3OiTSyCSiEn21ue0D0jQ4gmE8j29qIYKmHx+Wvx3M93Ip2O49GdP3KsI0r1HJMpaOHMcy5Ftd6OQ/dMqHXDe0ItrMBHaYCr+p1cXASYcrkKWk2OSikgqhLESP1il7l5wXx/orV9I0n0rS6jgSI48jrOrENItKWEPH4YSTWyhemiq+FMRWZtMHlVsf1IYwORNzjIyonvqWEsAwefmUayMoz2bLvUXRp/wllURLSdeICfrVLMI8t+OAUJ1G0X8m58qm1c/wwSqaTKF9a7HD+aaMugb3gQyXQbirEpLFzfh63btiFoENC0XNmDt3PRd97GpQ/yb+7agH+9dRciqXbEB1Yh0z+MkMa2WgYrT2sGQpJeqBSThxZXvG1UlbH+0OFvZTvI/1IPHPmNqwPI1Vi+t0nXRAIc6q85frLjSgoplkcuh/w5SF/hqNFU2id82zevmQp4PW2oiURPL3oe+Bq2f/6HCH3ndpHQ92YD5M9YhsKtv0M2mkAmlMBFj/wE5e5hPPGzLajnaa5dUCQ1T+SQasbZmVn93YvGreHvMwNbENq4nMlKI+1GQ/pgO+VN86g00bHImKKz7ufi1YPhYGMuxXACjWYVk9NPY+GiCvbtGsXE5AxCQVI/y2nsJHZQKKD3axmaHo8yRbQ+qWxjqVt1Nj38rASkGOXVKmsEOH7ZSiweWYQ0hQCKGrZYWKuaTM1cR9p7u0V5pMKkGqth6QUnYNOtO1VH7pq5DQ06BfIwSiScD1OAi175emx+chTl7UzVLavhYiLoM3/zkp9D5PHRVAAAIABJREFUp4tcvozpmYLmB0UTJikUGUGWrNaLrdfLGDwmgcXHN1DWfbU+Kj8r2WNjhw/bHF5NKgirPqbeli/2a/nypQzfmwyzYjGnTcwoqbajyjP6UYeQL06hsD2EcKFPw9nZzlLa67jEnhxRyuc0nEwRu1EXXTKdsdGnxFlY5tS5bqIxOW0wE+jq7UE8k0I004FkNoV0RxI9x0Yx1SphanTP/x5xRROu4/K3/Qtq6aVItfUjGFyJNg6n1oFYM3koe7bMwOTNZg40Kj/dxtWh7sBiZbX3pldwjTk5mZ8DyzEVBjSJ5jh34+tIsX5xUZmb0TNSlKI69UlEnEurYUXgTiT1gVpMK72W11EndVqFm4iuWobBX/4znv2LTwH3PcUGHKZTLTSuvxjPfeZrGEAaS//i1Vj7ib/Dk7dtRTCW0DhGtgE98drX2uS8au4YUVPnhC/k1dXjBKV4itPxr8wp8tU6pmdmdMKSlEEiBvusTBvVxxRbxaKELTQ+3Aha9SriqZ1YsaaKeKgs6h37wKGA9izk+LaQmy0hXwyjVGggN0NeM5HmrJwWuAClG43aOErdC01+sPmxjBocaBbUW1i3fDWWjyxR+nZk0XOBh1Auzmozd/b3ItPdhRBTxUQDx1y43m3cKLaP/xahFIeQtaHWIEhnM3hect4VeO7RA2jujaDJFoizH6J4wlM+2XfloUX/KY7YlKkc6/95jCRiEDxsuB76FkcwuLLGjrMOAx70Skk1k7Y213vl/UxzfKfAIS/xc5xkN8VQ3YNoTBY86hfX6PVF0X1Rm61RrqERaaKVr2F8WxmpSj/SiXYdJH4kjieAsF7kpA4uPTL8GPm5cYlTELASPiFyjQFz6jzEY4hlUkhmOhGKhdHe3YtwZx4DJyzBto1PooEjE+xfqIfLzz86lsd1H/4ZWul+pDv60eo7Fl19vXNBguWD8AWJC1gyEFU2uazfuPwzywWBpAQA78uulJ28UkOnqVV6Ic8hywS0eF2Pljas6sM6cMk0kVxczieJKhcOfXL0LEYTpteqsWWK5rpg82xpIpEWkte+Ah0fuR5bTrsBsckZ2ZYcStTQ9o4r8PSnv4W2/n5c9eB/YirfwrbfjKFUrDvU1lJu/39t4oYhyXxgU5OTc5pbXrCoi06ozfEOpUpF/5eLgxBiM8uWVlOEdZvDyptpaDqtJAJUC3n0DBzE4iWHETTZNqmiPduN2Rxnu9L6xc+9iciZQumO0iCgVongyae24YktE+hsa8dLTlyNZokzm2i6xkyag5pJajBTOKLe0SCMM9Ycj4V9i0w8r/voiKxNa+/0DPQi2dWJVjSO1EAWg2eswDP/tVXSuP2FB5FvHNbnIPGgs7NLm/HMc67Apkf3IThI5NSyFAlF3JgSHrTcdIVCWQdaqVzTxuXfE1kDznjYJZIRTZUbGGlH/6pZBGSOEbRzNjOkKNKOtlgqOWNyox1y7dAi1jIih54T4XXmdj4bJGupq6vXlVvUKhtphob/nH/M2c5BuYXn7plAX2IREsk04gn1H8xtRAcmMDs95TjMpgcmWMcNzWyBXtcCKmNUxaXNtYMlA3vA2XYh1vE0dbMVLH/pWmx9+hm0wjalns4f86eRKKMTs7CFH/33g7j5rr2IJPsQ6xpEZuEKRElEqVudTR67zBVZvzpCkApW9YCspFBP33GWVXrdk12hjWtOFRSJ/x+q3gPMrqu6Hl/39f5m3vTRSBo1ywXZwtjGTVRjU0LiNIwJoYQQev0IBPhB4pAAST4IhCRAICEGG+OAMTYG3LtwwZZlW12W1aWRps+83u7/W2ufM9J/SD5Lo5n37rv3nH32XnvttawuYA3qT1pfixKV5cnqeZpsAfFLBAUCGX70jyAP0y0BWnEBWiJza7jawAcV2g4Uy+Qy6PvJlxA95wzsO/c96NRrKHebmE220HzF2Xj8jofwzs99Hqs+/Pu494YtyNX7MDs7pw+biLnUx2kVMT3Se1OKRKLYRn7n5vMsMNZJfAisfSkOzrqWI3yk+Rlf2EV/vpajPXo2D0+JRm0RgwOzGF9zXAymUqlPXrOdjk1+kDRP1Jd9S35e0tZMo7gpggGnkaq1Lr76P7fLKPwL73kjwghPd05MBRpW57V+/8e/QaXDnzcw7LLz1uOVZ12OgfQqaRTziymjSc+GIm+k+0uIZ3JIjuTQf8F67PjZDkXo/TObUQmPazGTkNKhtWqng0tfcw32PnMCtQP0ljWmE+vpxWpZ78kFz40eCeKYmpxVKsnsl6OQQeKUAiiJGcm+EGs3NrH2jHORTvVgenIOM9PWDuLaq5TLOn0LhTwGBtNohgsoV2cwuzCrYQRpKVMhgzy5bohMIq9WDlUvyN6SxxXLB9jAvjIWyQpZfcxUONpI4sAjMxgsrUSUcEKXabOVaKJHkuBQLUuQ3VRKzKmDLadMljW7lUNMlWXyJVO5KFJ5km8515xGN9LES996AXY+fQiRxFEzaydV8zRzavKyaVVCpdA/ec830UivQyw3gMTYOErLlqPO9daoqw2kCTKK2JGYQvqoJl7dUEVomIuxELl5Q2sx3ptbp0F6r92rGOXsG22HGVDlGSB2ctqN0Hcdw8hrTqmWc/Uv0zqefhKdc8HBc3XjolDyRnYQFNNYvvVGnHx6D+p/9i/oBB3Mtqs4HJRR789joieNq/78/TjzbZfh7m9tRzxizBzJvTruLxehGDzauB0QgeVJQRYUjckYnZleefkWP0RAqp4AKfYrG3WlRwYYtKVswd83MXduFPZ7O4iHc1ix5llE0EQ0QdkTU/zgzK6BUVZfhQTMmm2107woPE+raDqOaBjB577xE8SSSfzNu9+IpCiR5nNDKR3K3PzXzQ/iZNnsTshsu+jMcVx+znqMJS9AKk5dq1Ou6gzHHCLPDfUjwtq6P4mxTedh283b1O88PP8kZhp7RSM0CZ60FEAuedU1OLm/hoW9DDIEEdPiSUsxkzTMas3UBVtdTE/Noc2gU29ogJ7WQZzJjSXjuPT1L8OhF4+jPksYihmWTU3RGZDrSzpRBAqlwUzP4yi6USKolA3i4DiF4aLI9sVR6Ith2fgAqpjHwuKsergMoDZ6xwzOQDrvGJmnxGu9hlatgVwhg+fv3QtMZpDL5Di6b0olmkIyjyDOR3uZGxmQU5FycUGzy9zArMN9y04kf6LfuV75KEXjSTSjLVzy5xfj2YePoTA4gw4WbUjFtW6k5qF6NIqp+Rr+/JM/ALJrECn2Iz++FsXSICo10i0bQpLbbI+xdFFj2IzePFCJjuEztq6szmVPOLgnty5coiJSBcBN4jDdtU3vZ0g4V2cu8s4T04mWmdQIh925tOUMHolqlItvQJ6a+LkEMVwqJL6zHNhMiLozWMTIk9dj5ye+iZ5fP6M0bbZdw57OLCbjHWz86/dhaPnZOOOq83D3N7aj2XQ2iWpSGynd6kPjLbMm40YyTSiL0kJK2bedm1OdSAofa7I6c9MuKZI1JNNpjeNR0VHAgUAvOy1JqjCSxjxWLt+FZHIRrWYUuQFOA+WRTGfUP83mehFNZJBO9yr7Y13IMRi6tFcX64ghjliGtWRELCe2ctKdBTQW66g1FlCj189iGeW5OTzy9Db85I57ZF7Nh3nhmWfhsgsGUWyvwmB0tdH+2Hohw0Ynbg9S/b2Ip3KIDHHjvhTP/OgZtUcOzG5GkJmS1jQRWva42dIbHH05BkqrcODRE5qMKZV6dA/lseRmUHkP58sV1KpNVBumQ3zixKRQ+J6+IkZGR9BpdhGViiUXgpOl5TnRNXcBtZpEYjGt4yRdHUSMoLyNjYAyZaSSf5tjXKxDmzU0W1W9ZrY/iUIpg9JwEYt1utVzGiqJeres0oIpIu1EQ2pDLwZ46vbnMZQeRoQqjqfRD2WiJu451TaJ6prtjQbVSUmNccyx4MYKTRObP5BKskWk0I1OsovL330pnvjVIQyt6CJIT9n6s/PMiSMAnWaI791wF25+YBJBbgSx/mXoXbNGrSt2MiSNxIyGpZqo2wTbDFOSzahcPKxzQ5SZ2YLkkZg2/ya7Zmke11tlcjNQVd3zkvnJhXKx9RM3JQZtZweoKBrQfyhktGVLKYZcYMPm/B0Spjkpw8hlBlDOe1cnfQTtP7gMy771Gex52ftQoNdqq4WZTh1PN6YwE29g0yc/jGUbLsbKS1fhl998TqmkSahyTtY2rPVBjXLJZj5JFFww4lG7vi3THqV+buHyz3wYhOHpm0OgiictR/AUDNhCaNYQTSSNjJEJcfErVmLjRSvQbLOma+PAzqOYmSrbYqi2kE1R7yiKsGISI2wruGdvi4Slgzxnjb8svnA0wCInVeJAIhUjrVW2KDz5Vm8cR74/jlvuuBVbH30c73zrJrTngebBBPoLg0orOxq/o0VKEem+HgSJNFKrchi79GXYcv2zmk+eaD6GVnDSdMUEfzHA0cN3A8654GXY9ZvDGgDoKZEKSjc9Iu3W+uKpu0jt5BA4Mb2ogMfxPhp0jwwPq1TyShNauM4ki382BcdT+timEMLRSJOo1dQPMRCJCLS1WHUSaR6Vvd6YNhb1t6xWZX/TCctziAANRBIN5IeyGH/JEJK9EWQzaWx7bCdmtkxLWYLXRsCS7cLFhXkro2j1kiDLy/qlTFs54pchcpzJ6DPJc8qpXcTjedWstVYL+WVZXPSWS/HgzduxfLwH0b6jStm9bKtknniX2028/69/gD3TRQT5fsRH1mBo9Rqx3yQWWG/pXspbOogiSnIJcxAe2Jovpv2qqZ3QOoeaYzLvZqr8y8IaJnYGOBnp1eRZ+IA9nN4JDWRgFKTjHFUfqFPbpfdMW4oTnF2MDfSojxjtzaEQTSI9U0P6yDzyQQyZ0Oh8nJYRYubSbTbc+3/+VUSWj2HqlZ9Eu07fmTbqQRf3Vo/gZLyOc173Rlz+rvdiYMMI7v72riUShyhyTppVrCanC8XZUpLjBbjJb9a0hfiBiWJyQc7PmbcP6WgLC2XUm019Dr4IEWcutlazo9bJ+o0rcOEr12Pn9p0oT7YR1uyz8D6xnrUpIPZR3KA2g0eap7YRWtjvkxwz+7BqrDMTIbhmmQNH+iIa/TObDNZiXMwiM3YB8owi2QbGNyzD6PIUtu16DJV9DfQ0ep1nr0V61qaF/l40IlEsu3gtCmeuxrM3PC/q4Ynm4+jEp0BCCjdmtVpXxJ+e6cNVV/8+nr99vzIgyu+QX8xgJuRW3NgoFqpVIcknpucwMXEC685YJy0yotAqExRALYAQPPNkeNaf/BmpX4hsQH0rcortz7JpbZtesNZFp6PhD9OHMoUSOfYRXHIqFaT8MSgzh0uojWYHB9dUPbKAtRcMoHdlEQ/+zz0oZcfUZ1YJ1+miTMlcotSSCWIJY4rTTJ954kZiEW1czUDnrBwR6huhxnGAMBrFqgvHsebyjbj/hucwtiqD9OgJE7d3Jy7/w4EI+m9d8bb/RCs9jGh+AMnlZ2B0fBUqi2VNSzUrJA41jeevxUv2FGm6DFIdySJHui1RfMlhR9vLP3UR/CK3WuCU1Afk0yrPQWkKS1ep00a920UlaGO2WUMtao6g6jG5FpDVwaxnzDE9xqFrJz/C18h0I0hH4lgWy6IYSyIZOFUL1obpOMa2/xQnvvsrdL95q8TXNHoWAPdWD+FgtIqRM8/FH//Dl5AYyuOB/96j9IqRh5uL1iCGIFvN42VkZeLklPK5eQhQsX7jKcs2kLxuKhW1fCq1hhBlL1zOh8yNhxTw2qsuw/TCNKYOLjDJVeZgGAAtNHgfTLGQIgIqDQJrpnMhSfxM8q4mvcLvg4GuZSNyGgM0QREbCm93kJdReFe1T1xjbUSYOYETWtssE2LVOT1Ysb4f9/74HqzIjZpCIqCZ6Gwhg0RPH0YuW43U6Bieuv5ZpHIJzGIrgtSihvQjEdaslvJue66B93z0A3jy5h1OEzpts8Ed6kIvuuujvUkTEycn8cKBg1i5YqUc8lhSeN66XxPcnDa4buqNavE6FwquBbLYGJj5/IxH3LTZU4eV6BmmUkpdGWDJ95ZAmsdV2I5r2SY2qVQ+AzMm1ymnLKmJVryG5WeMYt+2HcjHU8jSYocGZa0mUlQa0VohN7uDRq2KTIZa14biExPgNTAQcu1Qj4xkmVQui3YnwDmvX4++1Wvw4I+fx/CqNJKDxxCJkmtl+lpm1cryMYZXX/t9hJkCYoUR5FavR09pQCCdKaOw5SeKn+mVc+M252XIztOWtX/A8kLpLenGxD4I7gYIbi2sNQKGEdzEveTGSQdxVBp1nIw2MUPurWmfIqmFazrKS9QqH2nc3KoYGC4lJkZtNa21g3JNYFVhAL2kqEUjSF16NoZ/+E/YecF7UVqwi+XTboQdPFQ/jF1hGcNr1uOaf/4yOuk0nrzloBucj6lWJW1Pin6sq2NuAH1m1lJXV/96aRJ+wkq1opOWNR75rVTTr1IeRsyVhtQQudHGx1cglyfnloPzMRmDeWCNlpj8ko4SaXpk/lDGhkqGFDjPZMXSkayqZFFtgJs1HE87vo6EzCUI7mw2Q0OOBYRJQTIuphI/n5/AIkKpzglqaIV1XPGnL8Hdt9yJlclRbf54NonSYB/i2SLGXn0m2ukinrphO4r9GXQKL6IRmTUiP/2EZNbVwCN3H8Sn/uFzeOymbSLJcAHnC1nmfTpxzUY1wHylhv0HDyFTKKK/t+TorhD/WYEukXQaWoH0vCxAsGb0AweGigpEdKZfAozcZJml1bwvMZlUe4cBgWP8+SXdaYNdrP3H2VjzI+Z1erBK/K92oB5rM9bC8rF+zJ84jqBu4JQyApVPtJupoZDPaprLanCzRhFTjWoc7CqEXeTTBcxUaMaWxiV/fj7CRAFb7ziEvtUpBPn9CAPTuxaCrtMTuOmOh/Hft02ikyogPbgCpTVnIBZJSGmDa4EIcocEmnaIUqKMT73zYmr4c1uIl0ywkyi2tTg7CIRykx4bR/BTlypbBW99pHYsgulWAye7RBQ7iMaZf5skqRBChzKfcuezgWu/kUm+9kg0R/y0yZkO8KO5k3ptugcr0j1YdtPfIXbeRhy76MMA7SzYL2XWGQUerR3B0+0ZpHoG8Bf//m9IFHvx9O0HNMequpbNcg0RGMVNoEcyKVcCetMI/HLWi0x/+Vl403jaNSnG5cTOadZEA2NTKAReuvFcRWIbAneKjhyyd2OJGtVzXGcJBzBLIXc28JaTMQRqBcXkfMfIzmvU5FWbC8ycFzhL7IcvpGLoSAeLTu+Zi1kpu9LqhkYBqeIhPayQChJlXPGOjXjqV5tR7GaQySbQt2wZYqkcVl25AdVYBntvPwwkO8itnEGQqinCN+pmvcF0+ZYfPo5PfflvsPmGbTqJiEzLoiNus7tSWIwncOjYBKZn57Fs2YgWNFVPSLThBhKRIpdRqqzhCfnzWFamckQePmyFcTCCxAn2N40vzp4xNyazHdmZuhYjf1dOeU6CVTI2ak2ZionNDTEUOxkl9z4aLHAcAa/X3ApaGD9zGXZvfwb9qbTKGvZ3tWkLBQ0MMIMiw4knLj8D8QKtd7WDOFAQQQsxNLvAa95/GbY/fxRzuwMMrouind4nK1jvrMjnVq038fYP/ztmo+uVJqfHxjG4Yo0OPa4JAlKScquW8fl3vQwvG+uIO9Fg6h62lIFxuJ7bivxslQPEyEnw4b/dnFsZ8g9cSBwYrkZDrHvbZYitHdQbzE9NY37vFMon5zF/YgadahOpTgTRkG5trCtNbiTmoHBrHDGNNOULJsWqCEnlokwITYRZR4YBlmUKeN2ztyGaKeLkBR+20SaiZ4yo0QDPYhr3LRxGJJnDO772TQysW4Hf/uQFq6NkMs0hAecWHo8rdSNowt6t6k+mZE7xgBtcZPZWG1XJmjBOVKXcwE1o1Lw2zn3JBs3JaqyRtbEYLWZHYsMFjHiWuhC8oOuA5lCDCGoV61OK8x2Eiqqsr0j14wnPoELAwtd7YpS5YMATRUqHyaRc5zTepRSqo0XE01ejctTI4uxmvSYXt3pzFle+/Xzse2gbcok0hlau4NGLtW96KSqdBHbfcRCNbhXFNQuIpG3OlvIpqhEjcdzw7fvwqX/6NB67cQcyqYxOWzKcpCXVaGB+gQGti207d2F85SrVf2mmyOKoW/+fG3ChPCc9KA1exE1czqfEGoUk6OQ44/LHZb3veMT+AGC5Jj4yyQgajjd5UgUtAotyBDRPJrUc9Xwc0EYJHefP5AXhWOZ5FZZmt4GRtf2YOXEAyRqrQ9P/5qnL0pmBk319BlnOVpMwoqEHBV1rMTYaETTjIV7zwU14/O79qE5EkBo+iVr4InKFJOI06kqYYTlBrGs+9FN0C8sQ61mJwqp1KPYPihE4s7CAVq2CwSzw1Q+8DJn2CbTCONLxAMTAqVbC9hL9mdJZYggkpjBL4MFH87Ikgp8Ux2Xr2YgAx8MOfrZ4FN/83idVGPuWrRCuIDBt5GaI+vQiSqV+qSgsTM2ifGIOE3uOIqg1ETZa6Fa6CMj6cYbYUozgmzrDQyqusiJhsPzAoaeQ7EQxcf77VLtIwJORKBrBi9EKbp99Aa1YAtd88WtY/6rz8MD/7jRjKKKCBDlEljAgnqcAbzYfsCIaTwApVBhVkX+fmplCxGlmsd5imsxTPpVPo8h2Q3YQSal4nNa49yWA09vSInIOBamkqWtI3lSiZcY+4ukraRtOHXWMQM7711PgUD/5uMaE8WN9POW46TUiF1JQ3ZwHJCpXr5tmcYNlwYLb+AHm52dl07nxNWMI52dRjOQxtGI5EMthze9txGwZOHj/CTTDGlLLphGmKCzAUTe7H1y4P/nuw/joVz+BR37wHLLprMTuuIj5fjK5rlYxOTktOfO+npIR+cW+Ms1iZg9ybjxlNKH767+I5PpTV9pU5CzTKlTgH21gqExBNUdrvSnrYEYSjeh05vvwuTVqRH1NsZGDHiLfcPrKPVcOlXgvKNl0KA03l0cFOtbL7TY2vmIcL255Gj3JgvkIxRMS4FP/v9NRz93PQiel1mElEnu99VYMYT7Apr98Be65YReCZgyxZXPYvvMxDA33Yu2atejr71cZdPzkDP74Qz9CmCshXhxFduUqlPoHUG1UsTA7j8FYG9/4wIVIR2fQiUYws9jGkRNtPPfCIew6SKFCUugIUBpDgt2JFf0xrFpWwoYzhxH8b2FlGOuEeDxawS/a0+jEUvj7D1yNs84Y1QcR/Y8JO2+6G5aWiTQb4lT/Y9Rr2Ywsv2RMz0b7QhURDq9X6xqs539bE1Uszs5hbnIarVoXlU4d1z21RQPhBza8G3EaLsWJ3AV6/ZOJDn4+sxfzAbDp7R/BVe+7Gvf8cDuChlERefrZ3GzDjMbI8W22NIvJjXSUw/Ipeseamj0jMvu4JBdwfnZuYUFXTV7uyjUrUSxkEDZ52kQEtFGrin1SBhyCNVJb0KQGbTVa9j3q/AaBshPV2JmMo4+aMZgZejnfYKZ/i/NLUbkupcmOGv5kJ8kLlptdDnu06UxaPRiYFUVNG54tphSqlZp0hDmFM1s7ij+59jIs7JpC34oxBPE81r75fBw7UcPhRybRDpoorJpBM2Kc5obkYUkLTeOOG7fiw1/5OH53024BbMWegtQReR1MVXnSHzh4CIOlQQwMDGj2laCeKW+a9BAXt3yg6EecMraVBTcT5OM94ee0oGHEDKua+Lma+gt7zWqjuNaM/68X92Pq6Gei6w3bmMr2XOeDypVEavi+Xk6HAUW1sPrJZhxebi3g1VdehD1PbhZYyFQ5kTCROZUmEjKI6bkxW/MsQQFFiRwGzhjA+is34K4bdiEVTWLDVSW02mZETtYdA8Tc3Dweefx5fOE/70c30YPk4Cr0rlqHbD6DykIVuWgb33jfBszMTeF719+NPQu9aq12wizaLEVpGs5eD0k/ThPbm7tFKHbAdPq7uWXhb4MKHuLoFf1fIgE2jPfh/33kLeJZsk9IXS8lJBQN4/51Y2Q8+ZQGM/+P2ryrTXU4epYgU1pTcrFTQZFN96a0rchSIkXs9X/xWcQjOew+511IEYlNxkV2JwVsPt7FLdN7MB22sOrS1+Gd//Jp3PPD5xFWYyIPqL4Vq6QriF8mXS7FJLrMyMnWglQWnFUj02VOBFFqhbS+voE+jA70C43W4IAAD6tXKA2zxBJzJ6k3h2ZU5wJhb5btDqZ+THH9VI8GviWMZ20I9ZmdGsPC/KLSSvYbGeGloOioLkojvRgd0XOaPXMYvV4XGGfpvpFeOBNbq1ZQayziirechcb+eYyuWCVdzHV/eD4OHC3jhfuOotibRXr5CTSCOSG4YbuCarmG3r5+/OJHz+GDX/4YnvrJbqSTGfV8+/t7tQhZA56cncKhFw6jVOzVxpV3UoIgVsbKAVd+SPliadzRgpa8kJxgAfWrubl438yDmcGTQw8mSqBa2pVs2szOo9dcDttLhtu+zcTPLyqg0mMius490p2cDBjKxpzDngJMB1iszGGhMY+RoRCxWhcl9q2jduJ6mx1mEjIoo6+U27wMVJVGC2tfsQ6j563GPT/ei77eHoxdyL40Mw5qaidVcbc7EXz2S9/Bnb+bRJAZQmpsLfpXr5a4QHl6Du96wzjuuv1BHCxn0Y2aQAFT4EjUAoyoyQogRiVW1yEeQ8vZzqj99vO3vCn89+eewo7j80rReBrl48D/fu1TeohEUHliGY2R1WsEMTaDCc5EEppEKRX7kMwWjAXDiEqLCykXmJWJ0haCD+VF1Si84fVmFfFOB+e94VrEC33Y8ooPYHCyKlS7oxqpjXoigt/MvIiDYRmRvlH8zU3fxaN37kdnhhs3q7qT18wNzEXGB+4XjG/60+OGpywXDq+BYmDsPVebNSxbtgzFTEapsbxz2GoQsOK4yi6VVapKPqAUEu305P2gYiSV+WUKzjS909aG5EnFfpxqJKVwfsvMAAAgAElEQVTKrI8M9eSC6usr6d+46dRycEPTTN0ZeIiHCGGNxnTikTcrEQMnN0N63uz0jPF/K2VUqwvoWxdivNCLlWPr0GjGsOHai7H3wBwOPjqJUl8BtdwOpPIEQIDjR19AMplFqbcPv7hxBz78T5/Alpt3S962r6+oUUWO2c3Oz2F6fgZ9mX7kZE+yqDqcGQ1TN1E8eZKRZeXacX4+l6k4B+D5JZKFPIGdSbmb9eZn5Hog44nsNAZ31k/MMigqV6FwvVJjk9S1DWwAoszSvIWN3OxscwuHSNsJr00t72DLykh4oAZ1uTaH3qE4Tp7YjfHSiNJ/b5rOZ8uSRbJBZLWlqVNNSZsUFisVXPS2lyNa6MFjtx9E32ABwxvYozdRP1qqRoOkyspL3/ghLGIUieIo0ivWo3/VcnSbLRw7dAzh3CS6kSwiKQZz1sSWLfjxQ3M7sC9t0qXx19O+9+SN/xA+u/sgvvQfN1qNyRQ4AvzL59+PsZF+pAsFFOJ59GRzZq4cJOTnU919GIdvfRCpiRpirQCtiOkwsb4sNQIxbyS33WijFQvQoWp9xB6wTheO/kWjWP21jyJ5yfk4/NX/Ree/7kSE/jsBeZ6U34/hifljeCKYwUK1jU/98LtYrBWw73FaH9KuMo4ux8SoPEH5DzfMwM3Hv1MqlL0dyqUeP35cWkp8XYqDnH/ReZg/OYtChu0Mi+pSqHT1r2aTVSdZFjE3M6eNwpPGo5r8fjLJ09xmWEn898ytdov9R6NecjOSyUWQSX1OCagTOeSMqtV2xTz9hLpakETfuUm0gBIJnezeHlM9c0m+kjwxoxp0anYSzdgMXnXRWiwfWodqLcC5116MFw7NYebZBhKpCCZaD6MRziLoUG2pKetIBtX7f3kIH/rKJ7D5+q1IJTMYGh5AEJBAwpS4hrnZOfQVS0of5QoQYzCxe5FOmqQvN2ahmNMCkwome+y8p3QUiMdxgvO32gQcmrd/Y4uJwZZf1WrD8AgOs0fNq1g9cGk2n6I18Lmq3ylmElvipmjilTL9/LU5Kphel1h97FKwd85yo96U6+B8eRapUh25bheD2Z6l8sXPpMtrKZV0puP2XNkfvuKDV2L7jhkc3VHFslVFFFfPL302ri/yJCqtNl53zXUI08uRLC1HenwdSsOD6MxXsHPLVh0SsVQKMRcUlBI7PTYBul7uibO87A67coT1uqE51FW+6R/Dcq2Nj3/x69i06Qq87hWvxJrly5GqVTBz12/R2XscwZEpxJpdpCi3QhSWi0+9XIs0GrbvGOLpawJC2CJekwni9GHZ/mAkdjsXrW4bfVdegIF/+yxm7n8alQ98E22ieNTNZV4Ti+JAYx6/qh9CtQO89Qt/g/WbXosHfkiyAN+fpxJnNbnIynr4WuBy3DOJU/XhOmactFgpi0zx2t+7HJP7J5Gk8zd5xHSrkw2Iobka5eNwPRFOESVSSCVSJiymuo0zoQlDJWWBZLeTI4/8HUb/VDxp876UanGtEm8JyZ+VxpLukVH95mZmxDUmsslTtJAvGFgjw+cKkjJutv6lpYddCdNxU8zMTmO+OoU3v/4s9OeXoRWmsOGtl2D7zuNoHiZzDJio349uZEFpNgXIZ6Ym0Vfsx7anQ3zkKx/DIz96HoVsAcViFvk8gbEK9u55EaPLxjTN4wVEeL3SOdYEmPlIibXGvr3bbAqCTO2oXhE3v+AKaZMLiwqyslrRYL4NgdBPyRuGcXKKtaz6x+Q+M/X1/V63WW3w3U5gm5F2rbTTZIWZcUpUPWrcaG56Pj9+n6c7sYaZxTm0g2M4a3Q5MtGERu24ljzST2tSormsm0mznCrP4M2f+n384odb0F8cw9gZeXSyRzA5OYnJySnN15JnX2kA//i9R4H0CFL9K5EfPwO53iKObtuBxfl5pDJZxPjaMbo7OuNylRqm3qHzVlguZQad5KvLArXOeAo/f/t/hfmFNo7evwOTjzyDnmpHOsasW+Pqldqu91/EakwEnQLddnr6qQU+XG1cZy/CyMeWiixCNNnvcngLGvLabfVlcdbm76M9V8exqz5F2yGdtCzW20GI2XYdty7sxWzYwblvvApv+ZtP4/4f7bGBfuk/2QynGTTb4uHDZGvIs3EYwVmbd+MhNr35Amx9bCtKyX6zX6Qwmh6ODczzpDaFhLZR5UQggNo+PDG4qZge2khigGTKPVi1vgL1K0ny4O9wMUpkrWvADVM+LjKBTmxZKTW3jVivlDWr2kO+cSajFoiGxqVKccrSlEHSt4p4ijOVnjx5Agu1Gfz+G85BX2EE7SCNDW+5BFuePojudBKpeAwTzQfR7syZ92+jiXa9hhNHT2B+cgU+9o8fxb0/eAY9uQIy2Tj6+3oxMzuFWpmqjD3i+VqWxNPALCK1gLgpnCkVsw1D7g3x5896XjI/L0sE/js3r8Tb2PtlnSy/J1L6rBzj4mdgYGqr9hDnp52ihaW/RkYwn1pj6p1Od9XoJkkuRK3dz3gxRBJYTIaojmarjonpaVTbR9Gfi2Mk14NcIS91EqWstGXp7dW1skzgfHRQiuHyt70Kt3zndxgeGcNseyd+fuf1uPbaa5BMGn2SG/fhJ3bhB3fsR5AdRrJvBXI8cfuK2PrAQ0hn8qIFxxm4nfSP8AExv8wzyXVWrWRz3AdN5y0N1AQIHlp1WZgkYOEGdXkTk2SdRLqId4EW2xrgrKZXdDTNV40guRpQObgWIAegqV/rHP9MCnhJZ0onhtNf9qNK0WQC4w//B7rFAg5d/GEEtRYiBKjULgpQ6TRx59w+7A9rSA8N47M3/w8e+vkBdMuExTrIpvPaELIldBuDCLMhyTz1SGvsoN6u4aLXbMTBgweR7GTRqlcx0DfgVAbsQXHD+tqYf+fD4BfbD+w/q+6MUxzNUE2zrjSyvEYB6ffSqIs5RcoaU0WemN5xQMCDQ1RFPCM6TUmcRgP5bGZpookbeHzlSszNz6NDcoK4z+bB68GgmdkZG/RutzEzexLHThzDa16xEr25AQSJPM7+o4vw9O8OojObRC4dwzR+R9MPMdPKtQoa1TIWZhZw9IUiPvqlj+K+7z+JTCqHwaEeCabv3LsDq8fWIJUxQQKhuKSvpsxFnkGRQUci4uTyOkM4s/uwnrfpGlvQl8xrta6NwI0oUy4OprSYXvJpm9IF00ZmQCwzCGRqXWqEzwKcHywxhpJRHHkP/DXye2rPxR05hKi8K884LskMi1KxxEOIjs9WJ1DvnsBLhlcoaKaiCdXjXNK5QlG6VBymCNoRrL3yLORXDOPuG59D/8AIUkMHUGnPqvPAykrOjc06/vP6B/HYvgCR/DIkB1eiZ+U4svE4tj3xGHLFfs1gRwisatzTmQIwXXakFTk9SkbJdL90ODrZGpvkiyB4bOSCkLmzmQrZEc1tlzDW4lIU5QtJ7cJtUJv4M5sRRUSZe7kBYPVs7YubnI10bmhX3ToFgq7QaS7ske99FomLN+C5V38C2dmKgCARyAhUBQEemj+A59pzIof87a034unHJtE8mUWM9Q0nPNwQv1BhN963JGcTUrWxgqF1vQou8WYcsUQMhVxRtZTUPdyDZxTnBuHn5GmXSZPGZ20HnsBcOPwfr5kbyMQHyCWmf2qIYq6gHrMWdYcSLaS3LeqGciaYwUS9RYeAsg/LB2MuCHZ3fCosAbFuF7lMdqm9UXdzmyZqXlcdTDS2Vq9gfn4ar9y0GrlkEalsEev/6ELcf9cOYD6K5csHMRt5TlRJ8bbpbM/yodXBw/dO4+Of+wgevWkr0tmsfIlypTw2P/woXnLWOTZQTkIGTzFxj01xUKqMGiC36yZQaIi6Dbir1SNPZDt5xc12JwzLCdbTzBjUI03EBdBQmpWL0p/U8qJyLR1OMhmvm5vEXlM4iAsMzIJ4TRL386m8a2fa9BjUGzUKp1F8mTpPLUwjPdBBs3wCq3IjKknYseDPkPvNjIKOgCQcXfiXl+PI4TpeeGoSgyPDSI3slN4VT3c+V5VkzTr+4Tu/xY5JttPHkBhZjaHxlTiwbZumzRKZvKi2HDf0paWBbJY58rqYbfK+MEX3AVL9ZMe00+bVxnUnqMwTnAh1zGECPpIpHQmApEvd/MZUX46ImtIka6X4o15725v8OtaPT1/VdHepTPHj16D3L6/Gts9/F4W7n0eXyvOsYUTyCrG9MY2HascxG9bw0W99DdnhM7HjgSmZaVGs267B6hx+eN+096lvmKhj1dljqJ0gV5XSownzi2kwdbWRRQYWTaqIZ20ax5qPlCg4QRHbSOpZaqInKU4t68eeYo/olLJecWimVQx2Shjrpu5SLlNL5KkwMNinf7f3si//Hj7VXJxbRG9vr4CoQr6oIGR1HeVW6vqsrKXn5iawfl0By0dWIJZM49xrL8evbtmCYtCL/sEcFuO7KBJqI4bMJIjyV6t4+qkG/vBPr8azv96rdlCuJ4XesSzKxznwbm00qmbw3iiu63rtWZMRZpkJkXOr9atUzHQlk2rVGlH0viUQTlM6uieGMHswi5mMSpKWnaDKdCRiYJuXmAC/L0UMJ2jnUWX9V2xdu9c61V0KTZEEn0pzuoeKJJo4Yg8dXTHDphYn0QgP4yVDa5FLc+M6JJktwgQ7FnU0unW86TN/godu24OgkcHAaAnl+GOg7JJlXJZddFpVvO+6X6OaGEaydwXSy9aif2wUzz26Gf39A4ilMzppSSM1BQ4DvtgO4p89ocjfJ9IiPdXWmGGGnAdPLXu5Nq5OR9cz0kZw43Kn6lc7Rf3MrmDqUwerEFWfFnkyOVNE9TCdnIyG6ZneiN1k9R7TreKmjcj/5ycROVHBsT/4AkJasLuJGb7FyXYVt1b2Y7pbwUVv/j38+Ze+hF9/5xmErUByI0yrPEe1WOxR6snWij5kpIWL3nQODj5xDFE6kDurTJlTq/fLn+NpYO0ev1i5wRURXUnAFJjvIzUIjgemMzqdqVRhgZ8zk9YaUW2mE9k+nxHajVRB8gY3Ir9IuvCBj3PK3gyNi8UrU87NzGsUkWljJpMTpdOfSLZgu1goL2B6agIjQ1Gcf94GsZxecu2luPWm32Esvxz5YgTl+A50A+uVtrvUvapJA2pudhg9A8OYeHoGgwMDiOW7mJo9ieH8iGpQa8cwZbU2CVNWzchKLN1ojRokQFSsLvV/GVzabXMSiNiEFH+ezCWjjSY1tOExDwZHsqT4M5TvUYeAmAB72q5V5x3rBcy5AOrTaB0QmtKyUkQIshsEIW1QCDixBtrKMP0mv5oYAi06W00szM1gsvEiBrIJrBkYk2WNTjzO7VIzLR7H0IYhnP36C/Gr729Fqbcf/aM0VntCdS1benJdTGYwNXkC7/z8LxHmRhHvW47U8DgGR0ew9+ktKJJVxdOWjgsJTiNZhsD70GyTi2ClGfeSZwNKtsdbazqXS2WBW0Zfru3nj2058vEGOt1jc9WzNFoTREsypwR1bMSItYw0hAnXMy93spsEUsRNdv0ouRfoxvP/XQ+Q85lDJYze9w2kEgXsuewjoNUwwS+pOyBEA13cuLALk62qdJW/evdtuOfGPYg1yAv2UyVRpV48OUVamFtEtVvDm655FZ7Z/DyyyQwSbLS7E5k3SQU/f96JbJvyhbsXztBMCh1CJCmYVkY2m1MN6GsPDVArG7EbzM0t7eC2qX7wgVYWFxS1uWFtEZtIGiO737iq37xxmrtGKlTy/fj6DAILi1Wl3BxlPAWQUctpUdTHZHoeF23YgG4kjvPfuQn3/HwHBhJ9SOYC1DI7EEQoisfAydqwpfo5VTgXEweraB/rCkAZ3zCKY7snZNZlz6qjU4drgggwA5ykZyjy5nji0jB2QxzS+2Lv2g0fcMSEr8O61Zip1ttmj8bqO9akBgoKdCJgSe4320cJ07TW4LjqbFNT4cv4UT/7Hadppjcw6SANqstnmA4JnB5qOjM3Xrcx1BjcqTDZqDYwsXAUtfpRnLtmDfIpuiPwVEyimMuJQHTRuzYhjKVx1w1bsWzlOIL8EYTJSUQidr3iTXfaqHUDvOPTP0OQG0V0YBWKo+OIxUPMHJlAtm9AnRKbCIuKjimchLRWlWI2fMLRWj9wov3oWGgCsPT5Q9u4OgUdxO6lXsTY0H0I0abDPJFibl9fx0qmxrjBegAauHYCc6KuWWSkNaSLDEsnNL+/1CDniVssYPj2L6PS3499V30GqUqVk6+ajOjwwXY7uG1+L17sVNCMRPD3v7wJB7eHWDjYRk0Cb4YOU+jLZESZZDfwmj96FZ5/8lnkUgVNuzC4MLDwRlMwTSi0Nok9SC4e2o1ysRoZg4CKtSxIOuDgtcUt6znqlHdTLp7mp15mtQYuWHF9azWUeou6LvNqtTaG94IxQTbz1zVAoiPbDn5fPWNJqhiyXK/ZCKM15SOYm5s1KZhqBXPzM0gXFnHROeeh1uri5X/1Wtxx/e+wvGc50sUoKqltQMC+qaWq/Awc6B5ddwmeu/8wEtU8xjcOi0dbjPcYi8xbmDoqIe8zUXXSGvllFi0R3SNeL+WKfHvLVD5Dsxh13GbrRds9NwsWnqyUJDWgy6fdIrQwhXTaX+rLcrTSrRsCWkJYnTqkP5F4Xww45FqgTWdCyhFiWAmLYW+ZiLQJA+rnKB7XbGChXMbxyd1Yt6KEUjov76BcOidKJLOnTR+8Ant3nMSR58soUGu57wDaUng0NVQBYN0Odh+exRf+7QEE+VVIja5DaflqzE8fRqvaRLK3T9x5dll4/WQJ+iBH4pP65Kdlrr7T4Q9WtsqUHfP/nhq6QN5BYn84Lx+lYFKlt5tHaqLsIW0f6xdtusMI/qK2ufpORTSTNd93cv64Ek/jQ1JUMSKXAAYytXqyCN5xBXIf/DPsfc9XUdx2GKGrMcmkYozZPHsAT3RnpSzwse/+C7qFVdj36DxadfJjCSjZbCW/WLtcfNV52LF1J0ppRx7QWCEDvfWa2QKyFMsQZY+amqAYh7TrOiWLhaJtNvn/2KnK00AGWg0j2osUQMnXuBFBuCEqi1W1pPjgyfbhIjVE0NXMsjqpqHfL7wlkIpHekTG42LgZ/ICBwJ66aSHz9/h9gl8kQ1TrLczNTyGZncJF55yPVL6Is992Ee67/jkMl4aRzHTRzO9Bs0WXObsGRvf52VksO3MTnr3jKMbPXIG+oTwWDswikcqphSTwx1ExfW+T/GTW1MwseLKxx8375a1rFNYc51jZBck61YrWjW1cG7D3X6o36zZIUOrrXQpexAHIIdYGVWpLsoXJmfrSTkir62Dw2fN+SczeqbcYW40kDL+5DCBV8NagekcbmVRcDrdPTB7DzPx2XHDG2eZkkM4hmc0iSAa4/L2vxYO3bUdnIY7ScB/i/XvQCo07zo3rg/h/3nAXHtnZRrJnLaJDKzGy9gzs2vI4Sn0DiBd7FdxYz6ssEOEkpj5zwDlhmejBJta4R5bISjbUwnvpeRLBs6MXS3PK+wL5h8WXMHBF4PFSrcdvmK6ytoHzZ/HppRG0pUFMdUd56FqqpBNWEx2urcSGrUuXooko4meMYeDGr+DQz+9D4ut3oJUIbIiBvOVOB3vrM7i9ekA3+8Lfex2u/tsv4tH/3S+QhuR/EgsicdMzHjt7EEi2ML+/hnQuiUTEGFGGk9tMsdExzUTZQ+/sH9oYmRHjGQykc+TYTdrwrs3AB6bo6NJkntr8nAQ7uJDJhBK7hxGeSn6uByn5W6dgz3tNEoI3txapg7alAmH48MwHlq9LCmCrzkDH8bgWFhgcSPbnMECljoXyLMLISVx27gYUV4xi3ZvPxYPXb0OpNIBkpoV6ajc6odHzOBjBz0qlzNVnvxI//taD+PQ/vxeP/fQpFLI9qv3ls+PS/6UA59M0qydO8YOd+L0tNmOK8TPa6Wajn7z3XKD2/Lk2DMziZzMlDVsjptNt5RWvT1iHq/kM1OrqdbSAtTh58jeEa7B0s3LNnrMnZ3AjLAGObhSQPyHMgddIZYw2Qb46dh17DGsGSljZN4I412U8jdKaEi6+9hX45fe3Ih6hYF0PUNqNbruu4Rpz0ON67uJjf38zjpSTiBVWITG6BqvOWItdW55BaXgUAZlj5D+TlEIEmZvVMdKoeWYgccRQf5YFEac9zcNL/043DGJGAYKtIy8/JRbnTkneoBhrU4cE+5NCD1CkDIuYlmqae7g2tJN1JaTO2VprfViPkzef56wHVlg42AO1Af1EXwH9d/8rYtUu9r/hsyJ3sNdFyUve3JNhHbfM7kaVs4p9efzDnXfgwR/uQyZOXWVyUFvSpx1Y04uB0T6UJ+jDQqmUMvpKTP0c2OSmLeQzG7MmPReMQCWJiiVMnFojfM7KwguZuRPaVB1MTpWDF9x81BAyj1x7KP4UlxCBQ1k96YLXKxYPJYGc5QZrMVIifbrnF52eBetxPtBGS71QlgIsU7jJJyYmQLdDMoGmZvfglReci8L4CFZdcQ6e/PmLSNIwLdtGK/8iELAt09CDF4BDe8vsejzyqx141yf+EIc2T6gVR0BJ7BwnfSt0XsMbVOPIngZOmVay6XrZXK5lJ1zEhj1QRJ1fKgeEbVjqyr1FUIe/w03ja2Kesja/a6kjnw0BJVtHlk57tVCmzEKl5QYRA0XTddqTwdRsCzzk/WdQNVzFVFGMJmm5BK9loWxgGjf/8YXDSKcmsKa4BslsHKl4GmsvW491l2/EL777FDLZHEbGc6im9iDomqyqyeoyECziff/vFiyiB/He1YgNr5SiSKNcQaanF4l8QTRfL+fLtNnPWBN38Iw9May5lxzeYofOqUCnTb997NLQI1hEkj2rxxMqfCrp20I+yWFEYP/Nn2AOebBI1zUtYf2buzn8M8EQf9RbAmyRkUyeZUNDKP73p9A5ay12XPIh9FIbi0U8a0m2Gbot3HJyO04kO2iGdVx35x3Y8tAMwlmDzaS4H1vExks3YOaFGW0ioqZ8h9mZOZHmrTfm1SttzMu3I5jSSjZGd8gWmAm5mXyNMgbWbY5AwpuptFgqDVTEJ7BlWQi/eLIYD5kLlUHBojK9l7hYRNhfLKNUooyrnTys93p6Tuk6GzvLakL+TmWBKbLZiPhajekjpT752oeOPIerLtuIgTNXYPDiM/H4z3Yimy0gmW6gUzygul896oap53O079jJDI7snsc7Png1jj1xEulE2gUfA4P4VXWeQAwUlm055wtHDmDQ4joxYNBOTKs7Wb9aNqa6XrO1liG1HEXW+MWnnChIwOCz86eu3/Q8xetSyLDX8/8u7W6Bgk0paSylx9y8TlGS18UAGYtSY8oZRPOaXI3M+tK7O87MzePw7G9x9tBq9PYwkMbwpvf+HubbIZ781SH0DBWR7VtELXEMQViXtKwtGTLaGnj3Z3+GTqIfmcEzkBpbjemTxyTQx42bLPTYmJ6mfeLamL43K4MMch1cGaOSSlrShgdImCAwfWUNmm4feXl4qgi2qGSwtJvGcI1fqyu4QSxD0Wnj+r4Wu2yEzVpJdkrwxrHuM3DAjntLdwzU8GNUZGkN5IqIXv1ypD77V3juqk9gYLYhoriiI1sp3TYemD+AbcECupEQH/vRf6CDFTi0mT24kKIPeOklG/Di9gNIMd0KIwpCSkXCrto+kuVUe6PtLCdYn51Sm2AarDE0pb8eLLJUyNfmekpMs2ocjK8jX+BgudrmOn0NYQzQdhGfC4r3lAuaG5lUQ6tPTdJUJ4joeSbnygejf6OKQpVStTZULgvGtg3b8/e5IaSEz5Oi3cRiuY6F1hQuPWcIoy9Zhb7z1+PBm55BqYeDIh20Mnul9MCNR++g2mIFYTSFp5+aR7cM/NVn340dv9wlIkgu16P+NEE5kd4J7DEIOuKCyY8aCczKB/PbVe1GkobQ0oQGJnhSW2sLyOcKCmJ+Tla0x2x2qe+qk9hZ3XCteBMyOw1t8ovvytdMJ1Ogq55mmsnQ4sL3eINM2hg0TJOYJ7G3pzz9JNe6dVkin5ECcbWGQyc4mzyPlcOj4pxf/fE/wjNPHcXUoSb6B/oRG3oRYZScddbTxuASyFWp4z1fvBVBuojU0FmIJtNoR0IkMr3I9BQRTWfVnvHlmW1BZnYxE6B3Na31cO3z0J/JU3gpV2RYTATB7uWX+oPP0juS8qWImHNop+kpaac7cEWuB/Jk9U71tnT5u+rziQHiCnZaUbqJGp+WKgR4UEi1TQulbB4Lg1mM3fFvOPqVH6N962bz/KHyA8fx2i1sb81gc3NC0z1v/9cvYtXZr8JTP9uNdG8O6zesxuG9R3RTmIYnY0nN2JpfkW0QpkJyqKcJssbkLKAs8V4dWd1HdC4kXic3I3/HpFMa0olmmqcb7ni7ipCyhHSDCm5I3BQdrNerqB9ACLWsP93pLlTcUdx4GlEgTf1TaguTsU7pVf5OpS7wRWkfn4mUIpjutTA5PY9KdwEbz85j/CVrUdpwBn57yzbRGAv9ATrZF0z+1WlwVRfLCCNpPPrQBAYjWfzF378HT962HYl2QmqDYtPBTMD0rH0dq7TwNGacJqtaUr3wih0e+VTG0ek4i1XTRPZZhA+ACvSOJWSKkdbz5QnDTMfzc8mqUkakn3X2ma6OVr+eo6ZsIaq9ZKi9rlsaxca29wFTAcBlVabfXHNGajT/aqNaKWP/0d/h7BXLtH7e+sV34J5btiMV6UWxlEe3j8bW1F2O65mS+cZW4ez0At77d79AkMoimh1BrVHD0Mq1CHL9SHL6i1hL0vAWyxhs4yqbFe/aqJ3iO2jzdtGVbI2RMyRpIWvbLoLdY5cuORn4Rrnl7ZYGKyWkgqH3u3WbTm+oOsZACD4AzTA6cXR/QT5NUprqWiEmoO5qHd5URaEIYqU8Vt77bcw8sBUL190g7VsnbSTPmqPtMn5T2Y9y0MAbP/8hXHTlH+PuG7biyqs2Yd+Oo4iFEGXN4Hb2vCgVyjYCwR5OACUNBVwTb3QAACAASURBVBZTxdIbayNxkTjK2WnUQxMbM7IIPyNBEYmOU2vKjZx5fWhFezkeGEBC4gnvp05HTcLUMDg46OZ5rffosQJmAn7OV/e7YsLs2iDRmJ2ynHBp2YCBmDSRuGprkvZJAaSlRbnTwDkX5TA2MorSmWvwwM1bMTI0hHiuhjB3wG1cowmWFxYQRpJ46MHjOCM1inM2rcUZl16EF+7ag3KVxmj0ETIFCGPu0GjMaXA5Wqef3OF9phm2v07dM4chMHiaLA3rSjs9fGlgizO0ckjgyylfKqt5rT/MZ8ef4wZRf5ZC7sQiWM5wnJJ9Y4KhyugMe/FglzGv7NDxPV8/oWROF6HOH95v/l0Cdd0AR6cOIhudwdr1q3HFe9+Au36yE+lEHoWBJBKDvJfMTo3h5dtRB4+dxMe/fCei6TTiCTouVDEyfi6ifSMIqJsdT0i3mffJNqsRaLS33OGydDg60wD1fV1m1glNxlbFyu6xy2Wz6dnvYgG5WGARsKPepi0kk8Rc2pRehoQbXBMc5tInbWZPtnDRWUgjZTzZ4nBK9fwzazOeIkTQSvkChh7/Dqo7j2L2A9+0XJ7TKIyW7Q5muw3cVjuAxW4LL33HlXjt296HwexyPP6bXcgQhEmZUJdno4gho+a81Q6iw7m6kbWrXvi0TIJPXOkfb5T7XZIguEDYtuFDVt+NKQvTadce0qLUInR1BFt6ra5TyDCghikh081Oq24kFeatdFuv17UI1cAX5c9SS2YHZIEpqGh6hsCSSZuK/OECDBdQo9bA/OIC5soLuOLtG5GLhYiWhvDQT7diZNkoIqmT6KYOgw9eny/oyn40CJJ45rlpjAcrkUkmcOk1mxBms3jx1xOoo4pItItEGENIdQZZUHYQ7TozNUdL1MZjuuwGMvQZ2i2d1Nqg/kQ5je2kZ+ACuQKRo/rZgeG7ECxvjEHlBc2ZLtsYnAn4i4rqxAmWxvHcbDXXH19bBA43G670O8ZAaJJA3PAyg2sYgYanJw8RBt7JqWk8u+VuXPO+N+NlV7wcD/3sRbHC+saSqESft1ljR6Tgg2SgOnhsGp/8+p2IxTOI0Y4iFkHvygsR7+1Hh7PeZJLRtJxZmKWd+nzClVygs31oJ7F2JX/PeVOxzcl1J/R+z/JNp/IehxT7COVTItZporsJ6fPo8almsaKc4wsL0nZv6us3f4PVMA/ow5IU/Ywb2G5uG41uB8v7B1H4zT+hOVPD8WuvWxq3s/QOmGvV8IvafsxHWlh79cV4+0f/HlsfPILeZC+iEfbHDAkXgun6tdLn9Wn5Eo/YWhbyQfVyK6fxcDWvyeEAmkUXC0Zsd+LmYgZpUsoCgp/g8Owp3h+ioNXFiphRsiBh+8MRDKhW71Nj3ikuLO5BSqVaimj1Ne+3MaYog2qRWSqJAjSkD+vaSkTTG3rwi9VFnPfmcWRyUcxMtbHv8RMoDZQQpI6jGewz+F5JGXv0BDwCHDpYRW9lVMBNN9HBS990HgrLVmD3nftQmaUaYwJBzJU/zLAoYObKAx+whNTyfy7NzWSy+oy8h3SC8Pffja1YUD+dyHPa9JEvT5ip0AicbTCF09N+3nAS27Qee+Az47NgENSn5HpUIHTDIW6V83eNd22ZlhFvDPlWQHTWNvze0SOHMHxOGhe87gI8eOMOFHvyyA9XUYnss9aNzMpPHWS79h3DF75zP0BdKOIRuRzSw+chmu9FLEcNK27cuJzo6VniuQMKVk7myPxxA6XiKpe6xlPQHtAZbZs02Ltik1JlS1+WNrr+7ml9HjRQu8RB9aYaYVQvnzb7B8oTwvpN1nc6PV3236N8DE9Gr1xB1Hi4p4TBn34JtVQKU396HQLnym01UxQLrTpuLb+AmWQHF7/3arzkgj9A7UhWxHBq/LKSsVSsi2w2s+Rw5pFkf6O4WQmc8Ob4z6h0x/VVGY2LPTxhnU6wd2Vwo2QUaGMqafPHlkZazQTnWdRFf4lD8fYeZOH4E4DyJYywBvQYuYDXayoQnSWKHj+Hpm3o+sBUVSvXUmV+JZKkQrpB8m6AVDaDcrWMNVeNIozWcHxXGQefPYGh0UGEycPoRg6Ic8yNG+XIZtxE7SrTDVSOlBCPZZCkbUw2i9zqJM561UaUJ5vYvfkFBLWkVBl4DU2q7bsMw0zHHNWz01TdLz8mV9fq+p1mlB9/VOotewNPBNE2toXp5I7swCBK7Vp47nek6OgIPD4dt/64pY+MSQQM1cryPyuk36RX/X23zLGzJAdE8I3BVm1Luhh4NhuDcHYCG1+zEfddvwOFQgaF5VMod4/rkjWwIA65qaLs2HUU1/33g269A6WBMcQH1iOe70OHBtmprH6Hp2087daAH+tzhgOWevvDkWm8gZW6fxF/KAUIdoxcIuaUb9N4YMZQ5FPyofqg3KRuQkhC4K5G8RtXN9ydCL6INgc964fyQ/ovgjq8UaoJw1Ath95SCX3f/gSCdatw6PWfQqJtg/F6qEGA2UYZdy7sx/FUA+/73jcwfzyHZKtHahFcxAQZ1Bvk7zj4W5HX1ee8Po/kMoAwHVUEdEZT3pKT12u1sVHiuDgZufV9iZbbtBDracmKhAQ+TDyOBHUDUMzvxdIxN2rlepCkDfL7cQq7OxE73gu2pHif/KSJ+qcUQFetHrd5VV13c0kAT2qN7GV3A9TbC3jZn23Ai3v2oXqiiYkd82KlxQv7EUanjLhAxDcWaEiC6d7ciSlM76Xsar/xp1NZoy4mA/Ss6sP4xmUaQ6vXotj71CFUjs8h3o4DHZ6yvCd8RubiTqoFRQAJDPr6mOORzA70HGCnndYDw6ysVt2mk8gawSwG3axlE8qcLEngNYl+q6EGYytJh15kC1fDKkMhU6umZ677tZRJOdE5x5MXJuH48nwdM9kOsFit6NSWiigNrocyGDozhvv/bxcGh5ch0ks3yZrxn0m66YZuVrqNJ57Zj2/c9Fs0W1QETSJJadaBM5EoDSOeTCGayiKgeXgyBRYtTIE9wYbrm2uB18z+tIIz1w4F4pzwvxqSrssS7FnOGveUIJXfuKf/ly/CByFUWObXRqZYSkmcRrD6jS414c3kw6JQuPp6px/nLsbyPZQSqY61xTn89Q8iuPRlOPSGTyPXcmOCtO9otzCPJu6c34/Fnjiuu/NWbL5jL9JBj5QCeSOVUrgeIk2lWYP495WcqNNdVr2rVMren5uQ+lS+Ac5/07ifs+10B4K1Kpwxt5HuKXQW00A235ug1RKoFNhp7TeiT8WkHsJ6qlrR0IOXOl0qRVyNaKdGIIEzWb6I9GLfU3bkUkeiokRUCfxU81Vc/ofnY+fWgyjPVjC9awGZQgrJ3n0IIxxMMPUInrj5Ql4LfG5qAhM7ExjsWa9NyAkXm0VmfzSObjxALBVBcVUay8Z7kRjoRTpGzKOL6gJQmamgXWmhVWmjQqvQch1RyuxSmYQ92UxS/GaVMV0GNNNCZl0rE2s6CHAZkxK5pPllLTC/vvg81CEQJ4A1vu+XG+XWgoIBTHxG9P7VkL7zHGJ/l7PAqqdVG1Nvm1NLTlCO+obuvdXB4KQPSxwy/XozOOOSHvzmxi1YPj6Cbv556VJbu8okYw0TCbHrxZO47tu/QbPTFc85nutBduBshNmSAKsY0WZiAWSmxVNyP/AYAWEufg5+ziWlGAES1t9VOeJKFB1Ep29cf8r6k3aJLOFOTZNYNZ4rbxiNlJiqqLZxTCtLfE7l3F7027+mpQJ2CsoYiZQzUgMYvQCs+fjbkH7/n+C3V30UK8qGVMvXp93GRFjFXdVDaPQk8LXN92Pzz3ehlB50DB1rm0jIu1wG9YJ8veOjrrSgXL1gLQMzxubm42fSxpbVg33JOtJ5lRrybKm/r1dVL8m825zn/eSKofM8BZymFJlEro9NYopNv3A4gGbOXMhOtYH9YpeeG2pJdNrECHTiO/oogyhPNqZ3XOy9Pb1YqJWx8ZpzsfPp7Yi0E5hemMf0zjn09GcR79kDRMwzSUG03VJmwqBVWZzG/JE2wuoKFHIEw0iJTKAVcMwDSvOppdWlFZVLtSutefSvGEJxKIV8Xx7pfBbRHO9fwnSOSRqIJBSYEMRRW2hgenIetekayuWGetxBlfeS12IBlKNs3FynCRwqoPN/3IBMmy2F5J38/7P6bE0ZCGUDDKauweOWfV6eYr525ikrySKHJ9izshaNmXzYc+e9oa1KkIxi7aYSbvv+Zqw9p4ROcr+456daVoZL8HV27T+Ov/v2r9FodVHK9yCWzCPRuxpBth8R6pOls4hQNlifk9pqrsxkXe2YZsoKXWnFZ0X7Hz+UQIM67jdNtu1adlloub8tSH9TGA2NIma9MN0uQdTWC1SN4WoypsAk59uiMzqg0jn1Ak+dEl4ZQYigkzXh7zTCNuokm7ebGLzwbIze+GXsuu56pO/5HbKIo4Y2Yh3gueYUfls/jp1hFTc8cj8mJ7uoH+CiJwOqjXzBxL2Y8vLh+S99BqeeR+6sCOzJhNQdlEW0O0IUJZXqanuri63u0kkrzV87qWXYRITcyXiyhcAHL860U4VU0POMKC48ybSaayBTdD4UTkWRgC+dJFfHGVhCAIs6TbWlsUiJqUmPyaReI0EcKVJOM3GErS6CVUmc+fIVeOLmbSiN92KhXsb+LQcxPDIK5J7EYnlOWsFMfPK5rDYJwaN6dR7tSgUTe+LoyQ0hESfRnzO7fPYkgiRtskbsMT5jprRc9xyuoMMhrVhsjI/3Rsg50WvNvtaRHo6iry+P4dF+JEdz3McSGuc2iVLHmeJGHa6TuPrU88cWcfIwjb5NkysRMIvhZ66ArhEm4UJDL6bCMcQ6PHVN75ubnjRVM++y9cr/cdZXgoZKnwlW8tQzQUGfkUnFhYGCZQm1lN3maQYNnP+Gs/DzH9yP5WvaaOOkNg/XNv/LLEvYSLWKk9OL+OCXb0Y0bKGY60cYTSJfGkMrKCJSKCHd04c2a13SOpPmwct619x0A/XOI27dKlsjRTgw+1hPA1VZ6lFlY07ZLK1P7yzyGnOJNYvnzmo40X2JrNF2ekhNytMw728q6nok9RTwZULPnm3jidR8DTrz8QM02EboyWHNfd9GcLyCfW/5HNJBTJukFQnxeOUYtrSn8UR3AX/x0Q/gvR/7azx77wtIVFKYq82ikKd9hkVcooJ8L30212wn15csGm5Y3ghGVd83830/RTmv8+NaHYymBCwYjNQPTtKGkekigTDrQYvwH7OUlgHPExf483QmYG47MTGpxc9eMOs4WXW6WtvkbjquF26iawoiAv8MOCTvV7hAIq4WXZXDC+0Welf1Y9Ur+vHsXS8g1kgikgWG1w7hvv97BP3DGSy0NqO3VNQzpCwLhc15zby28sIcuvUqKrNNLB7LIZPqRyRISXybJ6icnzhS5wYA+JyqlbptaJU/VMCgxI+lpmq9OcDKwDtiGDzpjW5AlFQTWgku1FCDIaneqFT+ewd60bOsoPtLjCKR5eB+KCPz+myIykwV5dkqZidm0W0Q/DSZ1zgoHMishOyziAzCtZ516pLRRz9gBlujD+oEk3KFUU3ZA1I7jrPCGnInRx4IYyHWvXwEyVwCv7zxYYyuqiAar+nAUvD0znyO8joztYh3f+ZbiKX7rL4mFyKWQ7JnJbrJAuLZAiKZNBLpHCIJU9mQwoWE+LtC4Bk0/PS7AN6E9bo9wKqSgJnToXWvC/2mtDrWC3QZUmrtnVMCzR4GFxTvQAFLv6y/JFKDyDCWzrB48b1TkhL0ZwlVGxeYIA0F6ViTVlmUR9rYcNM/o7VuFfa/5qPItQKxk7qxCO6fexG7oxVsCWtYfebZ+Nev/TsGz16LrffsQWe6g1jKUGJDeS0rsGsw5zfOufaV+k0e1G1mX8uLtkeXP9eK8emw/7zkFfNFOdhuQe5Uz5GR3TjAHCs0CiPfn5tX4Iy8ZiuiKdoQvtExfSrD96BAnI3HiVi6BOiJI622Bnu7bTGomMqSUdWNtHHGprXIroxg29070C1nEUsZCj20oYSHf/Y0cv0ziGWO61kxmPb09iKbzmjRzM7OmIl1bRELs9PolNtYPFFEMtqLbpAAurzOtE5go23SGI6v46RiHFAiJ8S2pbFKIU+b42UdZ+uLt8aGyPVcQDqsDYiE7BU71h6d51lmtMIGFluLKPZmMDw2gFRfCsX+IlL5JHJFyr8YZhHpRNCqAfOTZSzMlrG4WAWn7VqLvG/UvzJ1RD6QWo3WKXQ/NOcLtdt4vXSld2L46VwG0STQP9aH1ecNqwW3/cnDmDo5gdzAIR1ZrMoFIjmwVevfWZ1UG8DXvns7Xji6oEDRDRNID64BkgVE4hlEklnJ10Sp501AjJkWNyuzJ1JGZcPqZsV5rQQAHWnII/PKfk9s+P1Q5G9q87imtk4hl+Kq1nNpkicJeLjeCn3H63UHsf7ON3cMXl9fGrvE+KMaIXQSI0JOUVedSznWWrOF9de8HvnPvxc7r/0ickendaM4QHXf9D4NGdzTnkY0XcQ3PvY1jJ03hjWXnoVaO4bdjxxApBJHrEVU2VQVuJGpjMHTdXhoSKemUn1GOIdYE5klt5arq1JbVBptTCjr9Zlqvnn8iEXlfl8b1IEjmgoSPbKNSr0mLi1V/0I29Li4iJYWcmhUjV/MhyCvXFdfM/DZAo8gQo2neErvX+8wXSaS3EKWCov0xmnX0bd2GGsuLCFsdfD4T/c4+46I5GKDWBK5lUls/uUWjK2bA2LzOvXUVuDMaqVGvwCEHTuhpLjI0qfeQKOyiJ/8cgv+ZNOfIuykEYTkc9sAQUvSvIZxcNNVax41tyF1lgE8pSnnw40u2mHcZkltOsurXri5Zke24L3RhtCpbkP6BNx860snE0dFHQrMcoRrqFybRyIXYmT1AMbWjaBvpBfJBIfFI8JiVK86HTLZhEgVzEAv9r0F+vAanK+xDioYxbbdaOD5hw8gbMZkU3L05GGkSy+awFMkoplkG4K3TIIBlfz4Q4eO4Hs334VnDtQZwsUviCRLyJQG0QwyOmkTGQ5+5MWkYk+XG5Y6VAK5JMrIAKmIgxgzFr4SueKntUeDF9ddGeYyabUdZGTlFiWPa388nw4w+UFsq+GMZaTC34EB4ipTv8lNZ3he8hIBwZ2EJlRudXEzbFgPNuyiGQ0RGy7i7Nv+Dfu+/n9I3/GkHlol0sEDs/txMt7Br7uzaIQB/v1jX0dvzxC6yS4GVpew4iXjiGRJK4sDrSjCJk8HXorxO1WzO41nMbJ8K2JphNF1FEXP7qJdZ5pm6gmcYZWSvJArO8m9eBdBllq1jaBMd/MG5mcW6djp2kldDUb3FovKNDrOJoW9Py4Cj4h2OObogBciz/Qt6ka6ohISACr055HuzyKVjyDIdNCttrBt8x5M7KtiqKdfgYenMp9LMhtDelkCd//sAZz9stC0puQcaCVEX28vjh4+gBgBNPka2wLn14kjB/GVb92iAY8zlq3HZedfiuH+lRrcCEO2sKz25yYNWKN1CM5YSs+U2tzzbCZW7cMo2WZ+3paoadK1x4zAYJ2KU3JBasdKrMCsX4mae0cIBVN3UAiLWQI5+WfTV2q362h36+hwTakHamm3viJsxcSRpH1KlHW4PSNtPjG5KDnEv0dRyPShHdBDKI1Sfxbl9hGE8UOmONKwA4G1NF//FJ7BPv4ifnTrA7h/60nbuNEUooksOpEU4mwPpfOIJXNANI0wFkUik9WwPliOsDxJmCg781kebrId4FbzksgOXwr2jb8mZORh9OBp5E9IRk6fTnLj+pTR+LvuPjjqmT74aRxlGfY6Rgk9hITeOoTWvE5PQdsCHtp127QUCIuFmE408erHbkJ11xFMfvBfEWu2cDLWxmOLRzCR6OD29oxO6He96R14xXmvRiKSQSxIKlK2Ig0E8QCZXFILvo0W4im7uUbnNObREmLOWiYamjGx5nEtbbHxPa/9w5TqlEoGvWH4JURaEzG8f2l0YvTR5YJzkx3qJSt51vuKJ+3IzUorHbXN0HzdeaGd5plGlhlXVhP1Kqd/aqhNLWBxsoGTB+YR6SaRjtLhjqbSRYFC2ggdo0SeaNBs+RDa4aJOr76eXm0C2Xa0OavcUrbACO8VGRKpFF7ctR1f/96v5AgnlROWPd0Qf/eZD2J2ahbxsB8B8ohHc4jHUgKXCPYws+CJKlAwZJukJblVugOIEqna0thewh0o5ytDcvOrEndX/GS3Gdg7d/RO8aQjhgxLTldahqwJiXSzlWQIPrEYvk6jabPOtAzxd1aWrG7diePsABdDn03RhFx29li7aKGnj1NfZFIxbW5henEPXagta5CAuRt6d84XGnSwxjJuu+cJ3HTvHgfwkdGXQDeSQDeaQoqbN0GQLiOnSyLNiVxRzz1wptogW44ySdpfUQ3fc237+WhlxIdWXxUKgiZClzAdYZ2gblLDn7AexJH+r++XuBpSJAueRg6V9pFRQIqTqVEqtiTqxdVgabbQSKncGfBSjbYwv3IAZ97wJQzGsnj+jR9HqtXGweos9qKMnYk6HqjNoBW20Zsfwpc/8LfIxPvRbXQQxqzWjCdipmFEBQ2nB9QmQZ99uyXhdvrmGhjEyOz1kj3t0IgWdhLwzzwBTe7HNHB5UhCgoP8rTzI1z9VfNAQwlkgtSalSgzmItJHJxhBJnZJtYaYh4I3AXtuE7DRZFdCexCRRO23LaAxEsTpI0rJqZ5mNZ4qqGZx06obIkPUTi+BE/UEgUlZfUPYligbmEGAC7yYxRBK7mFnsgycS2PnsNnzj+7+wWVG3mXLZND7/6b8wDnWtrs/FINBX6Ee7TiQ2jk4zC3SziEeLrn4n+GVtQipJiG0V5Wlrk00Bec8aZOHUi9W7PKlZtrCmlqE4gdEEHQrpR2TXw3tPwzdNn7khA6G8zpuIa4oTPv5w4X3jdVsZQvle8+ONJ4nSG1bBHrOCClNsAVdRAxejATKFJOa7m4GIlXnqtWbTSv1tHt0sWYzV1ZY964nFDj7wxesRTWTUOgqjaWWBNghFz6AC4pkehPEUYsksujECVQES6SwLGGV3IYOGRNJDeRglSP10bUNlity41uqhKJshhNLuWSS7x3pnVsSbgrpa356f6Taxd7iTlKk0h4xkoO+zfhEiSpZSzKlBOjE5L7XJfq5DqKvxDpqXno2+T1yLwtgwDvzBZ5CaqeBQewEHIzXcWz2KZ2ki1m2qyf937/scVvasAuIpuQcqlWIrIEqxO474uTYWWwhSUDDgbH6e+kskHKSM8K6Nau0MEUm0qU3DyPvWaqjemTl7gomxxY1q6cUD9G/OrZ3pFEESD2bF4m5mmUikhgusD9jsniLmE120wXFj5lg7xtBFD1Aw0MlqlKlVOqkNyZ+hoF09mEYjtUsqItq0Lr3nHDQXkhhITZqLdRFo8H3psMeTv30cP/zZwzrx/cZljfeRv3qLpchNow6yDUIsQwqP0k2i/lIMC3OLiHTSaNS4+eJIJ0tIxqkYGbfgGjJQMEAJ8zeBcmY8HGSQjxNJElaOkAyi1pSzDeH7MtUnF1rMKUer1byqgpzxvokb0ErVNpMJ2BsKTJDKSiRxoCUxy9vRQYp/56ZN2iy0PWumI3XMdx93oJGVh0K83bPjuuHPk7TBzUfLzocefwb/+qPfoRkhVZHrikMaZHExFYsDHOiPctMWkMwVIUVutk5V8yYcvZHkHQY1m7xiNsQ9qq4PD8MD46/TIL2QPjfGxmjDWoZEAd40W6RWH3qlC5EWPHFen8XYUUuULOcd4/Sil5QTtJmdsJw2uU5p46BqwDroIv6ZazD01jdKxXD6+tsxd9N9mOlWcaRTwewlq/D9Bx5U/s9ToTeSw3Xv/yKyhT6kYvbw+H0pChCdcywtcn6lcOhoY6rR2Cek4DVrFvXPDNP1LSwf4bSxGk1kc3kbR+w0zb2BKWCEFhxMobgZSOE0tQKbG7RJmWj8FDPNNqoRMrQAOKSeiCuFVbsmlUaHYmeOyCL+ruOu8nc1OkfyhZwBTAlSp7Bn/rRbqCdeRLxQA8u709li1BLmRXHThkw7WUe5z2ttszbu+tVvcMf9z4mkwV3Az7tixSjeee0b1DZJxpm+2eepafiE7x+XM4Iye55gDHydDmamZ6V8yB47NyxlhlpNysxkEA2LCNjUDSOIhkl02taPVXbTNuEBS51toF4sK2czyu9z2oqGb5wgUtargX/7GTHf3IwvFwNPcUmcUpeM7TeXjrOeFHU3ABKphDZHPJ0QOMn1zM9WDXejHhxUIObr83kR+SXzjVRbOtAvOvBTfOlYBB/7xGcx3RlGNdqLWCSp+6PWFdefDAWIHrP2TiCMJHTopLJ5taH47/9fW+8BZmlVZf3vG+vWrRw6QneTBQYVHRUJOuo3I8YZFUEx66goKDkjsYkCDTRIFgUEkSAqCGIYdRQwIIIISu5cXTndujl8z2/tc273//985YPdXXXr3vc97zk7rL322gwDS+nnlIsSKhGx3yMOoeh3ZPcPtGKfojFqIjTtxgeusFlT04LguRL57dqO4kYP5AAvtTg8TghIDTPSBymoi3ARYPTIDtJBwVpSyK81bPlvr7KRF161aqtmuf4he+HTJ1u5UbMtzYrlv/RWu+0nj9jf141Zg4OTSNs+O+1jX3r/J6yne9AbYJgTaoifR9DCrwFrjaaRqHGaTMCDzDjAJmTZrZnUG4MH5uDJqMlwRbV5B1WElAcBPH5WLkFIcLYXG0rN99JXinxpVz9wiw56CuPGmTDq9y370Gcvv7iaJOyhaFjZeC71YlZUGaUlfrPSSvVhdFgyW7J654uW6wYN9snyQmlbXG9d18uhFN0XD5xwMYHYW3vHrT+wJ558SYYvigS8ad/X2Pvfe4B6jCnfSRAAY5HBA3pzgZd4PNJSxMakwqJL2mgNYCwJ0S7q/rlu0H4R9MFWkgmbnJgUXpFJ9zGhzVL1y/y6HwAAIABJREFUTrN6v9YE701JLZPuslKZweCUtEgZyGNTojDiacm7iQoU/QlHcEWXUqmiFjkw4FoNdpLz7om4cE3ZbEJiABrfyhC9dCepprVyz1ijWVSFgByYlBCvifH0PNsrEDJ8taaNT8zYcSeebOmOfivl97FmGvZTlzSaLQmZBcOPYcrK8xLxNJkhjfgx15/rsFy+X/zubDavWdHqFmVSvUYf+H+JDasObkUScyXMXIkhL6CV2FDBI0YChbsL/3ISfkr0NuUxyoucNyqGh6Q6PTSGu+FRG8OeXAmwrWEsQY2mpT+wvy0657P2l7cdaZkdBm3VDafZ4x/5mnWUKjbS0bTmx/axzlyPffP6222qxJhtl4x5/35vs4P23d/6csstkcxLJZ7jK/qbRN0CgyvkuKJ9qvGBHMebsrlf5TzhcHGt3AeHFMMFwUI5OShqmO7HnNoIuPB9Ne8HNQiXbM1aMsiPKD8C/NAEc0Jy583y+xpwFQAsKSHEBmtNf4jAjfNjVW/X2ru6RI5wLJG0SmvW8ssnrZ4oW7az03JJJ+YrjggjWAmXNWmC6QREDu2pp8z6Kdn13/q2vfTqhDY4HVx8ffKwD9juuy4R8KYG+UxabKRCaOogQvN72jbHKUZTrF+sKDh32HnpGuoVBPoQiuf9eN8yRAmVV7ps6+iYLVm0g6YRZixv1WpDOTSH1yxjzToN9DQ05ARMcV+kN/CfAXZoXRTIKu1jmH6UCEO0E5r6FWJrzErWevsGLJFCsYW8c8ES+VetXJ2wzs4eJ8dkMzq8rXRWDRuUGDu7GRA+oAFt1VLdjjvhRJuaXWAcgaV6d7VCcrElWlnhR0KXpS4CoEk3G4AUDQ3h8JIDE3FIi5zSXpdl8p3WkevU/bglotRllti86/taUR6k3fcY8gANuQ6eJ+Y7ejSxKyjU5QTgBEE15/N6o7MeHlY9jF5EfS+WUvBwEgoK7CbqWQtLu23lPRfYlnt+YYVLvi9v0H3fBbb1+4/Y1I8esblF3db48GtULx0vVOzKm+9WEg903pdJ2wfecZAI7r3di9TMvFBJ2pLh5daX77bezn4RCogGsGztHAkgJBIHQqnB64aAQR42x3owhwSkNBDUnEIXROB8spzrbkUxNRk9dSo54uvyr2EMpNDnbfNxMWSy3FJGCLNz9L2QB+sgU7pxZJBpBXwWXoxQvNwat6W7t0RwTyMrCkDHbCQJAzipXymPAMG6NWsVhbEwmmRLBTA27ao119q6DUi9Wps/fvYZx1omSU6cFmod66tKRwJSLCMdpFecNBLeNxArFH1BtkFzStMJ3BjyOjWuBG0yRWgQIrX2TStXSpYipUh3WXdvh02MT1mxVFDDAqEu6U5P92Kq0daRzlujlrZmnTIVOXbKki244DCmcqEkaNZqJK1Uqemw8nwi4T+XT6nubNkZa6TGLJllVnLShocHbW521lMjvDaeMzDdxMuGmVUq2ab1I3be6gvlQYnkrrxmrX3jkttsrJjzHBcvrlZqB7UQKEDhJEFKB91L3VLqnpfHTeIMldfCwmKfIn2TEVKf2LDy3Tq4nps55ByZIO4cnT0lVYmga8ufPDCmA0TPKog+kCviQ3PAJgh3ydM5isyXI4d1a0EYqDatvHjYdvjZ+bbwlxdt9PMXWa1W8gHXHz/ABj/+YXvmE0dbaZ9lVn3rjtaRzgps+P0fn7Cf/vbvEkFLJ1J26H8ebDsOdlulVrHRqSn7ya+fCMqLQqiUO+XSHfaFD/67dXUusVymV/cFcum9sRwkV6NQqCpUzw2Qiv/UJhM+psS5o4B+7oFwTmxqDoka3mWQ3EJXar6JfVZRUSQIb3DwvAljIFG2MFA7lekUKOb5l/NiNa6TcIuylXJgKBQVG5sesVvvW2uXrDlLlEHCdcA3RRNBJsbfO+TNQmKhpTI/CO/mHl9pS6Nql152nY1PzIu8oKjIzL76pcNt0ZI+AS3VMmNMaPwvWk9Pv0Jf1irqZeu9Ei40KNlWoopAOIH0QH4psC/pAgc+LdGnUYisH0j0GPt8vlOMNxmFMP2PAxJbM2nw6EOZpMUYWGRo8cQcCed7K3SnqQMZWqYaVOr20AO/s6mpiu20bDdbvnilZTJdajKYmhux10JvzBeF1itqKpdCAwkH0eVk4bk3NMKlYV3qKOMMEIWZrV59qW0am1KE9G/veJt94pOHCYD7yhm3WLHZa0lEBQC1WhlLZ7g+b5CnPV4TDpizVKPu7g39hEmIxXFWUmlem2yPn01sXHVwK7a/uXV2TxDDYB3S0J4WgSQXqHY1x1gmwkT7wXfBK6G57nv0ED3E9AXhSwghsXu5bvbZf7eBr33YRn/6Oyt84zuWalat1KhaK52x6V0HbOdrzrKnDznW0oe90cqD3knhIFHTrrzxThtfQFKlZZ2plh313x+3cmneRka22s8f+7vVSGCouQUADkNy9Gc+ZP0D/SpBqLUrge4zfOOSUNcowQqIA7qraXoJDh3IZNpaVY/5+X42xxBqJ65kssiXcvhZP8JuR4Ep6WgtABViCCxEPkjdaJVcA8tbCYPUjvS4XNpFggPNhm3ZvMme/efzVmnVbLbARPWmGFYnnXGMLVm21IaGBnWdAvqkEBEGlyn4cjCwUa/I4HCASWXaoEerYasvuMLGJuYUVcgAJxK25pJvmCUrVipWrFIuquXP1RvrXquVfKQ/b0UW8V5DtSK+fyy7qQElGEepVgRsRfcYSl/CAEI0wH2o9Bb0uXU4SUPCVADQZxEUQq0YOVRE40HUWXOEzhFWoL570YVX2eZN04YIP4CVcI1Wy978pjfaRw55V1t0XDKv9arQZxBjUiL0onxNMCTegJJN422rNjszZxdfdoPqtRiQq9eusc7OjD366ON2y3e+bTa4r5XTSy2R7LSmDqU3FERD53xlBUHWEM8Aznc4i4jo06sF15oDzjVv3uk9LZgtCmEDDUBaSm01gqDIGObCbl/XBVSIobSTWNw7RQ6o8rSgNuBaVds2CWB183W72ZKLv2z1xXlbf8r11nr4cWuiHs7JBNxKJm2yp2W73LPGfn/lWut+80orUzMLnkSDnusNu3jtbVZRIGe21y7L7D/etp+V5mbs4f/9q03ME9pGzVqTNTv9a5+1VtMbDBQ5AAjkctJIjhxnvBQHUOUX1au91KB8jUhB+TxgCG16jvyyMVmfSLrHKLCJhJsjiwrpQU7ca9gCIeH/8vfQOkk47fvVDzC9uL5RWlarLNjzL75sv/7V0wq5sEllapbNlh1x5BH2uje8wRotn0b3///yFkG8d0rv44d32yRB1iGZaNk3zrrYpmeckM+9otB54XnHqwcVcKi/t8d7mBvetxrr/qrZB5X+uCElBk/Yx9wjPLV4uH5YolfTBIJQEhPfuwpiT4Tns4UiCBijvIijRDIHNWzX8Mqonu31bmicTsaQvG8I4zHMZ5xxkVUqAFYJNcNw+EGM/+tD77bXv34n6+vp13NCk8taSOs6FRUGkz6bZ0GRJtT3wQF434VCyZ57caM9/ue/2gc/+J/2tgPeaplswi688Ju2dWSzdaQ6rdq1yuazK6ya7vNGnGDoVM1JYLS9RIaFVfOKhOadtAPSzIZRmEz0tGW397dU2lGZxEO6qObHxtIhbHioHBdN7p3NEaQ6faO41i7lH9BILaAGbLUsn0haIVUXwpy1rI0N523n606x1I6DNvO3F+wfXzrfBsoJ6yDcTDlaizebt7LNZLO26q4z7YU//84qNc93/OFnFK7NzEzYP9aN2b0P/14PIJNs2pGfOcxymbr99ann7HdPQ1NzwEglK0valz9zqK1aOqAGb5DcwcEh3Tebzw9MnLVLmQrShiPpURfa4xsvX4kwobEbnrtiqWmfYwOCYMuC8qlhc8awLzZpyHNrTKWLmwnND03aMUWJ10bP6sYN6+znD/9eD1Oc2kbLyvWavf9D/2n/9q53tsPKWBVo52J054SculGc87qr5uY4SAcVMZlu2WmnXGAzHNwUYFXN9nnta+zzn/1ooDnWhAADRnHQi0VvZ9REwoWFNuIdUXBeV6b3NsizAA5JjzuE5tG4xDq5YyUOXqkc1nA5XJEnQsqFkwF0WrR4kXdKpTM2NzdrOcpDon0CInUoraEWy570mnenAKTTTrkwpC2OHWBkcQDHn3iEDQzkBGIymRGVDQxbjJTm52a0p1XHD/wDFxwEXUcDu2StTIdSld1228tq9YqcwAknnGLJRsu6u1E3SdlcJWkL2QFrDPyLNRLeiy0pJbfVIqwANMpwJiCw8HlEE+TB7ky0h0Zf85/AAG04P6KlEagSmpbyZBzrIxJGQD2jNZP8SMo3Pkajo9qyUqppKRQsyM2olQ50Wd+h/8c6Pv52a+Sy1nh+nf35xDXWu2HaOgiRMklJ1TToP1T9sGXVZMPG/nWJ1d/zWsnAuEay1495oFwrG4b2tkd++yd74rn1eigrhnvs0P/8d2tWq/ade/9HCvCx3xVA4F0HvtH23nUHW7FyRXuwFpZfPbsingfeqiyrh/o+jdDXKW5MdVKJk+tKDIpZAlPLJ+wBvhASbScuH9IQFp+NHME68jDE5eSJ4yC1MHlBZQc1MSRt8+aN9qN7HxaAwUEEZClWy/aGN7/JPvOFz7cxBO2D0Jboid82AKgyP2OVYqFN4eW6kbKZm5+y1eeusVIZTB5/nrKDDnqzvffgg5yjWy5Zd75L9++dVC0bGxsTe4swlwNIIwYGNWppd1ALRe0j2+GkmJD/ekNBRgeK94pfhPBKDXgeQWhBIX/CVEJiMBpjVYRIB9aXk/Pxslmxqij7eT856VTDyRnNhgQWzjvnCgdnE16S8464uq0+/1SrVGbV0IEoHNMPCaHFvZc6p0eXfG7/4IDNzxeUg09Nzcgrwo5Dfobcvb9vUPf76KOP2YMPPiIwFRwFeqeUK5Mm9tTXTz3Nnnl+zH7+u2etmuxRyZP7zFLfFo+acBlHiJF2aqpKhOyxrXt8UG42InyxHuetWWF2DhBjyMFizushoqOf8soa7NywCt4tlbfGULelX7eTdb/3QOveb2+rZxNWL8zbyJ+ets1X32d9r45Zg+6UVMsytTDs2qOENkd6pitplSMOtHKiYnXxNgHQOLx+XRC6YymHDpNLrvq2lZuEl2Zf/eInLNtYsO/e80uroiKhPl0ecMpWLem1zx7+YXV0KB8MaLKoiiGP8dw9KCuQW4mM79ROHz/p+Q7ibz7Eyr0qG9jZWA68ONjgTQmx3hdTCT+4/uVGMciqBE8QsYE445Ue2OnpMbvz9nusWfPaYZl5Qo2aLVu1wo478QTPo8OwMJDbOJ+Jkgj1ZeiD9QpNEOTyPlyK1/f09Nr4xIgf3FLTWkmogg372Mc+bG964x5+YDS20g/cyMiILVmyqL1+3HdsPyMHjjREMmuRIljj4DW3XwcOffTWREDkjJHKiPeNzkFSMmGWkFjeQWxO5TFAPRUBhNK01TKIIiCqCJgSaSNvxxx9ZqjJO0OKEg+G+vQzjrUEWEeSCAK1EPSrnRG3bcZuRc+X+49RhI82wYgmbL4wKwB02bKVVpgv2SWXfFPItvSypOjZtIVGRVHCRz7yETvgwP2UBnEQy7Wm/fXFMXv06Y326pY5a7Xy8rKNZMPBMHXree1ZSP6WPT6g+6UpQPUkTS5rqd0IF69NhwIFAARehTfBK6FG0D9opXzScsO9lt53b0vvu7P1vWE3a0JHROkBAGTrlI3+5Vl74eYf2cCWCUvXmpbBgoiUHtkgnuxHaZLYjTT5nl1t+rWDCr9J2Fl8wrLYi6m+23TW5/dIkydpN996p+2//wG2bLjPuvId9sivfmMvbZxTWx4sp0SyaR2plJ175jHKVfEO1PrQMJYqY8aBoFhjxkPIy6sjxkGVTJDWRLMpJ3kWz1lbLZeEAQkFuo/AHd7AvbUr9XMgvfHCQzXPD32wlw4j9cFORxwhDhB68/1KdcFSiQ77/f8+Zk8/8fcAfDWsSG0y32GXXHZpmDcTR4iGubNBwRLomzzXieh1q5aKYqoRTUDIGBndYFeuudWKiLgHIbavHvkZ6+/zaQYeaTCipNump6Y0FnN8fMyFC8JYFU+pXF1C9yvlCTfGiA9EA+b32Gld+bzNzsy6sEGpqCYPfhaNIx5GgntCrr27yc27A1QKH5NoeJUsq95hNrP/DmGlS/Y2rb9/wDZvHbXV513Vlqd1XnvWVq1Ybp/93OHaG5AcYrmLkBnecFWySt5LrnUI/bdxSh+lrpjrM2iMa5iZXrDrvnWzJZNZGUX6zXlNVbX3nJ122slq+O/tdVGFqenxtjh6odK0YqVp9/3qeXt+S9GmFlrWQjkDZU6xv+qWGNnjgy1CMMJJVIYWmg1LQ+1LmJV6MpZfscRSb9jd8rvvaLmVSyw52G/Jzow1QOUysEV8kjj/y82WbeOTz9qGX/zWEk9vsNx0yTLFqjXSZpk6OXQ9dAGR7AddWno7s3SZBMoknpuSSm/Wip95k82kK9JdwjPyoFm8uQLMGTaBWXffgA6Kt5Wh0le0cpWQrttKxYL9+S9/sz8/s6mtbkC4lkulbPU5xznNkFJFBklOZzl10zNbZtSHz3SN+SchICEX5Q/Kz4R3YgIVGG7sWldcKCwf6S2HDhYMDRzwKFmjRosgi+LSrp6zcCgoNThzykN195z00GZF0MhSOrOUbR0Zsx/cfo8sOb9XrbZsslywK69eK/pjDOXFtQ3IcIUh0uWSIgcpKyh3Z/zGgkLCeq1iU9NjdsXl31EDg2eZSTv55CMtnXZ1TAAfNQJIZM37ZQuFBa3bkkWLdI08lwLicFLmN+Xh8sahCYBDENVBkEzlIGfDNEKEyksLBT1jhrSNEoYDOIn5tU0TTOURFDxqNevt65PHJiVD4havqq7aIDKPfI5SmUbTXl6/3m6+8S4dZmq3KgV2dNiH/+sDtudeu8i4w8FWGsOYmS5C4cmQLjniLYMRokz2zczsjOfBoU2UfURU9sjDv7G/Pvl3HUxNWgy6VGTNr33d3nbwe95l9TrGpsN2WL7cJiemvZEeIK9WtGwiq8aCucKs1ROdNjLWtJ//+Vl7ZbRu89Zjicm7H2hl+rots+OwZXbocxK0OvcJo5qWZLQDOlOlqhUnZqw4PmGFZ1+16rqtNr9ui1Vf2GT5essyADpYA3GAE+qrTVVduUI8ZCB1SbHAYnIKV8yXQQHdUnqiPtOTsspn32YLncyLQYXR66hsHhXwo8wLaHjKNWdzHZ3KK5B5RWVidOuIVYolW795iz34iydDkd+nHCQaLfvmxWfoUPK7CwvzwSPkdIidoOJhr8TQOVzBa3Ko0VjicIjHvb3MrIZGeV0T1DSyn7hXCbABPqElHco11DhjmByBKZHVU7mgtJgXM4rrUSN6kvpx1qbGp+zG625p85OrlYZNFgt23U3Xa21iGCe5sEACATBsVEGSg/QJoTlaX+UFKxYWlMNNz4zZVVfe5m12ut+UnXHmcd4QENacziLWgC8iFbwjBg0pHQ4sX52dNEl4VEHLJlEN3pZD4ioZfvDcM7fkwbhvgUWZtA42/8ZYi0KriY7uob1P12ca43HRv8bgOSHfQVS6wHg23jCDyob3mj/x1JN2//2/CGqWPpWQ8P70U08ytlK9XtHBJWTnQzNpIqKsTU5NKoUSSxA0GK/ZRe5e9AaRQOGN0xtY/8suuVa8AOZE8QBJigTCZdJ23PFfs3QGz+nenCiCz5EKB6owRHFBuB5RORDnUrloOaLBWkrhf2Ju3dOtRKFszfmyFbaO2PzzG2z2n+utsnGTNcamLQ90XvN2JuW8tGSFso/mnQSqIIOs1QGDtwn0t9gGFSelCUmNyhPqg3RVBcKiTpC1tNnL6ZrdWt9k//3lj1oyBz+1oBwml3cAJDJusGoKM7p7dCDiYGEeNCijxHGaTXv2uX/YAw//2SoisGdU68tlknbc146wFSuWtjVx2QnaJELWyUfTVizhdX0mTSQ16MDCOop6VMGbxFolHgwAAtlOVSbaA5uh3/nnx+kKeE8JxakU41PpIRiwebhXjd4gfWm1rI+pgPB+az6i8/qrr7VEM2nZdE6o6VRx3q656QZvRQylJZL9tnEMqDYHq1YpSeGhiQepl2xiYtx6u/M2OrbVrrry1qDVxBpk7JjjviSkXrV9zQRyCiiHj9p2rL2io8XGXLJkiU1MTbjxDqJt5K2E0vLAGimSF/WP+wYU09CtZErfx3vG0lKt7lMN+Wx6a9nc1Mw70WzSHF6vZPjfnf/b3d3lhieTViSmAW8yFFn74X0/tl//+n8dmMphBLxF89zVJ2ssCXk841kgzfC7maR3xnnpzjW2eXZ9vd02NTWlZ0sEpucnkgwRUNNefHGD3X3Xj+VICO9pKPAGiabtuc9u9vGPHyrwy1NPP08Ab3FWcmSjOcbhyqS+5kgCe5SSeG6PtwsKVfse6ozUEUVXdM8oUCGIyIlYEb6ilKWHZZENtY18gcV2fSHPdfiSWnxoKxOoxWGSQkHT5rIp+21y2h7LVNV1ctzXP23lwoxyP5DCyelpdYSwwdkkbHDQxu31o8i5uCnQTz5306ZNCqXuue9X9uK6rQpRIXV3pBP2mcMPsX/919fJikt8K1Abe7p7tOHkeekU1fDk7YTBlB46M0oWMqhO8Dr/ooxCCcOHNbdVNxDOzuVUQBe3JzBj4uKomSMYxO4er5UK4Q80SgwDh1bheXHB7rj1eza6ecxy2bzyp9ly0a6++QYrl/zBik4phNytOmR4WX7CZO6rUra56Rkb6u+2mekJEU82btxs1157m8+HSpjE3b961OfE12G9o4ER2URytH6v8kKI/pUrAvyQ5CFHdxpnwuhKwqty3RxSIeSphO200yob2bpVLLA4VMw1rb03Soqhkjjy0ZzbaKo+xlPU1bBm8IsLCz5cnIHogHA77rijQl0OELjNjTfcbM8++091FZGeYYzz+R47+9wT5Ol0LyIh4bmzNjc14cZCpT0veymCiXTe0LvuP3fmE3nyfff81Na9ujk0X8AdcGNKmnH8ScdIXkh2MJwnnlds1pCoXWjMiHs7dq1JXIEvDu7fd3l7S1aFsC/U9IDO1U8r+UpnSMnbhhm4PhOU/CUucuhOidKRQdlBnxFqwRqiFUTW+D7vV0iYbUxV7c82axtyLWuB8taqNl8u25v22MkOfPt+uiHCRQgQ3CAT75jAjuedmpy0TsoMCcJaNk2XvFFvLzKkjNPskKLjn578h11z/d0CJeh3xOO+86C32CGH/Jdeo4bqQCBwEAjrTtO3o67Sygo1bl8PBxpUXwxsp8ikicin5sCGecB8hq83qDRtW2HMYmjUj6FtDGtl4cXEIkzyMN1HZjiSzAb+1c9+YX/+wxPSLyY8nq+V7AtfPcL23nufYFSo/XmPq64tWHYRSAANaxWrV2rWrKF1PKcG/C1bR+3SS66VvCpe/i1v2c8Ofu/bVbNeWCjKiGZTaZuemRGxnnv0JndXT6SWyWu6uvOKFiIqTq6D2J4a+ANnm9fxO/wuh0jN6LxPB7N4UbtwkbyYctAJDnjFmvhasx5+cJU/57tEOxSpRs7AmzHUxighw7RdftkVMk6u1AEWkbRlS3ewI7/+Oe0Xyb2GUidhf7JJia7Te8nTSf3J/YpNTg7c0+1lsXAu8p3dViov2FVrblTLIt6fL5whTm+XXXaxQw77EPRkPQNO1PaOh3uSgQ57UVUGxoeKiaeub/f+mOAnV+wvBQyNDNmuTqlDGw5mRNO0ELh39ROzeg7wYVFSWB+K62yMhtecKImQm/Lgs8m0zTYqVutIWWrVYivsucieWZixB37/uKwPYIFarMIcWcCco796uA4PIbl3eqRs6bJlsv6O/BGqzCssZTMPLxpqgyIgeXScIEX6ysYNdu7qa62JymDSB2qtXLXcTj7xCOtI5iybY+yDK1q4z0zooWB1NOM1rIUsv8Izn1zo9V1XamANfZN5eAXgw0NwZNkR8RgWubfmMHmOGz1tO3pRLdhJJuoECaqP4q4GttfLL71sd91xr6WYUl5vWalet30POtA+efgn2yUUNTyEkp6Xspz9QxkOnrLVncIIQLJ164jNTM/bNWtv8vJW0+wrR33ZBob6LUekEuIJs5r6pNUvqwPheeXM7JyQ20gsiQO4AXySrIU2IdEAtVWXtVUzvlKUvA5ftiNjC0Fz2mv52wZno52t5pagEaWy5XaypdK7Ar+AaqoSl6tYoMpJOMuzuvTSK2xkZNQVP+T10/aW/d5oH/3oh937yXt75KNUp4bCSF4RF3I/7DkcCRRNwtply5bbxo2uQ6W5SY2Kbdo4bnffdb91dOa1z7jGBdDyjk779KcOs/7hPpdI6uiwhdkZvYb1Y9+7MD8sDJ/J7KIPoSQLkh0ObfvgeumD2l0gGQQ5mfbBDQQAWQNCXWlMIS3kaLQCZaRbRHxvWj3RsGZ3hw5poydrXTsu1t+ruy62Yp4e06QtTM9ZpVy323/8U1kVeMOIVZMPiNFUqdgXP3+IDfR2WblGWJyQFacPE4V58kg2zfTMhKw23+/M5W10dLQ9e2bz5k120IFvs5nCjJ1x5hqbmCyo3MB9dHXn7MLVp1pvvkfavpoWD8ocvK3fO0iqN1XH/IwHyn+RqhgPrkJdqX94Ez3kBCeLeHPCtoPrDClZ0TAwTQIFgeIWYiEPP4M4t09m93wsHtz5uQW77JI1AlDUcNBoWe+yxXbGmWfrWtVmp3JJLEU5G00IbzphCzNTVizMyIsNDw9pzX7/u8ftlpvv1OGrNZt27upzLNvhhzaWSBhDRxrQle+yufnZdhrEYY8jVLlGNjyhJZUEvDkGItFsiNwwPT2jZ0Zk5GQJb6cEwALRlv5ZKMl5bTuMlgxhMT+L6UA0hrl8t68nayREPtS5ywBOXgM+66zzbG6WecKu48R6nHTy8bbNwWmqAAAgAElEQVTHbjvb2PiYT2+kbioEuGEtkPhwPaXinMpy3NPs9JRyV6538+bNiuqUE2dS9u2bb7NyyaRdRaQoDKBRs4HBAfvCFz6pzq/ubk+FIndcVYWg8SZCShFcB/qnt4xGFpw0wMKA7sSTK/d35hT/C7pRgme2G5YVaV78EuPsherKEzSsmEtasi9vM4MZm+1MWKMvZ4munKV7UCQEmnc3T7jXSieso5W0JkwUelvmS/abR/9s6zZPhPpgr1WqrrqByv5++/2LHfDmfUUOTwf4HlTW5VOj+FjgkKYResuKuQNwwGKA6BFi1Vslu/CSG+yFFzaKLcRCQB6/5MLTESG0RDpq/3rYFVMBGRKQbMm8OpLpBBXnJgtICdPzZP2V6/ng6HSH82SVF0ZBdhD3KNcjHV5y3RD+BtJ6BCZ8j9Jp40oeYglJRdEbJiDqX/7NK9XBIpwgkTJY2ZddtbZdP465UvTokigNk80b1bL0lCdGt9pAf78Oyy9+8Su7796HZEQofFxw4WobHO63uXkH3Pj9DjWsu+ffOjqqTQuvl3VgPRjclksnbX7ePTAhfnFuzhqAKxna4jyEZeojXkXjV6gpKyUCw/DSGOuIlxUoKgka9lAct+kgl7P5/J6kl0bomWH2jk9713NGUUTPqmDnnH2+Vcre9+yAUtouu/xiGRfRDquw8ZjMkFMoXFVJ0D17MuGcZb4Qkfd+aq+5x9IXf7/xhu9IUL6js1v7gSiO/fXJT33ChgZICXx+kaobNKyEFEZaz6HfV6qkgVYcS4UukO8OUljNn1btTzFGVrWaBJpPqkgvACKMOaynTPKoGbxfZ8LSOw5bZcWAVXqYMNC0Enlp0JnFIuFBgemxQjQnk89I+yfwnRU+ohvVqNvk5JT95IHfWJ2ByTnGUThyCsCUyrTsy/99uAAgWtpU9gHgSbvYF1azo8NHHPKzwWFU+BMmnWg2BS1lTXpgG/bkX5+ya2+8y8OrdEpDmc5ffaZlMjWf7RsOXDLrVEIeOkwlQvToIWUs2sOsIdlT6vASyPZfHiIH30mdMhA2hH6HAeGANF0AY9IiJszzsJqNKHazcno2Laiq52SIrZFSeD9x07598y326qsbVQeVbEAyYZdec3V7M/D4I5LP1cQcmmiJjQzIt3nDK1ZamNdY0J8++HP76UO/0rNHB+rKtWsFVM7Ozckjo1jB78SRK+R3ceNFD0hqUi/7QVe/q5kMqBpCirOiHgqdpuUTAQMqDYp2+Dc9q573aW5wkGfNh1nBUs9QJxGlFUgyPgiN92Y/aDhYGPzm+sxuhAnrp6dn7dxzz3ckmoMIut+RtYsuOl9MOxpNpECCXnMBbe2MJH6IxNi/1JcVNaEXXXO6LV/sryg88be//dN+8chvJHkjrx+ihaHBXvvoYR+wTqIXqZsglMeM3EhqaVl3l3tz4R3pjMJm1fzDJM34HCNnPvHHnd7cwtPy0DPNhC1Y3aqZhFUHOq1/r50ttWzQios6bKZZM+vqsJRKCPhLn/ZO6xGAUnFmTjfCDBUAGG6SBwBXlUXhQuK0MR2erIeCExMT9rv/fcKm50loIIZ3akwI1rhaL9tZZxxv1qhYoeggCP8pf8h3yqry/s4VLdvKVTvpYKmpXZPbQCPr0oJCauTo486S5ebmUfM/7ZTjbcnifpVFWEwsp5DYdNqe/+fztu8b/lVhqELHunNWI7I+PTOt2T+AYpE2mZVkTigBCb111g6GUGUwjXRxcEHzlkLfJz+LpAQeFrVr79bi4MY8mfAOPSQUIFnPhP3pj3+xe+75odg+tIpRq117443tvBlvHRk98br0WVnXqtq8ZbO8R193p8Cq226/yx7/w5P6/XRnxk465RRFMOwN6qHkwXEEJmvERoNGOTMza3vusYfPBgboq1VEzKDEQTPDYL+TZGCW8ewJOVkqjBesN6K7GBoDAsE+Ep4SZtDyORFoEodZHGSK+97dJcE5rpnwVwbXx5FieNl35KCFhaKdfsZZDsIS6WQyttPOq+yYY76mKIz8ER0pDNj4OBEg+6aivcs9VUpFb2EEoKOVr1jUGm4fyn/rmpusXKyLp43KhWZEJZP20UM+YCtXLRWSrxwWOR3uLxBvyHdhyEUBOtdjdsCP/aIDLCDO8ReF0D//xCEtDqmhDtiXs3R3p7WyKUH7XT3dWox0i1EIiGjCrmqoN1HaRaG/dH52ToyoqExIo7dCmHTa8l3dbe+NvjEbnwslb9V8n0TCRrZM2e9+/5RALjGOArm8VK7Y2w58k711v9fpYLF5RLKoVq2/H7JI2nKdPfJaGJHFixZ7eNZqKnf76xN/sl123lldSRzcY084x8pIodJHm8nY+973H/aB9x3c9m4sipBO6o5SE3QtJaGjgafsltZDajYbQnGxtxS0efsDIotMbTvwmmWwwgQ1IdUB3o80Ov1uQPCrNe+KifmNpD3xEhm0f/PWnc/bhvWbhZSqFlqpaDzIFdddGxQPGS7shiSGlfF6+O7gwKA8VKVcsPmZadu4Yb3dccf3VYME61i0dLGdedaZAlbmCgVDXoaNxf3iDWP0gAfmGivhcPmwNUf0ObxEFYipwWQDvOEZahpElDYys6WLh0SiIMWhTMSG17jJYPw9WnMRPkJuIiRI/YpaNMDc95rTTltieLH5yUHZXzxH+mVPPe0M77flNR05e8c7/s0+8MH3e5seTQjzc0oFXC8Mj1uRMdLhpSxYKstg4JW5Z54/pSUiBwz5zTd9zzoynS5HKxS8rNz2S1883OqNsgw468PaCMRUq6x7Zp4vh5k1rtBRFSYVOlaRUmqnUme4hsTdV50gVDnmWq6P7GR6nwgeWDRhrqjC0DBqMlLAiO2xevwZ65E6BNKHNRsaGvJJbqGJXu6e0LzKFPaWHvAjj/zOKlXCVAJF16SqVetCHo86+tPWCrNyya+XLFtm1RrT2wGuvM7a09trvb0Dbs3xbI2GPfDAA/aOtx1oiRY6S027/Kqr7U9/edYyGebpJuwtb36TffmI/3a1ytD8r4I5qJ7a9OLwMsZpOgMGSwuQoCl1msCHd2H+q5MouG4HojwfkuVvxfIPyGWwoGrf2zbdnVBRHTTybhkh4gJhNNoyFMI1tCorgkAuD/GkaeecdV7IP/01qy+71PqHBkNrpQOlMe/2afF1MaW4xl133VVtkYBGk6Njdvmaq2z9xhFFJa/Za0/74hFf8p7QdFoHi+aBXKeP3fBD5uioDkJob4zElMgG0kFGqI/QmQYOt2xG+BtLTGAlDgjVrYqGV5D4ZSN3d3XJ6GYyQe5Xapo+j2lsfNzXDGYZ1Cf1EGMQzdcII0FzQb5bA9fOOWe1vJy8cCppRx51pDrEmF5I9MM1k8viff05IgnQtMIsA+U6bWZmRocMCdresM+Q16GL6re/edQe/+MTCnmlJ8UggEbNPv3pw2zvvXe16WmQeL4f21aJHreN/4yht3L60EEmkC6kEBhOTZlkgDhVi/uuObkVw1qFs6F1T4AMlEAU9rarAUoJPygS8HssUHTnvG5qckoW0KmECzYwNKRifDzQcVwjUphefmlpmNWr6zbbU0+jLuiWqMyhltSF2XEnfjGoaTi6uXjJUt00KoPk1gIzmi3r6xvUweUQR34s+QjhWrVcst/+/jH7zq3f10hHCuWrVq2y8847r93gz/06Z5q65YKsMNQ28qVysabQT8oP9Zo2sTYh4Av86HLRXnrhBVuxYoUsJyGfT1v3QrsAIrE6nSmjNY1lJrxPoiUghTxLXGV5fS/bOLnDSzTpVDYwqqB55u3Ms86xwpzLw/J12nnn2bIdd0Beyz9bAE4YKRkIIXgtrpEQdGCwVyDMb375P/bjHz9gY5N0ppj9x3vebfsfdID1glXMzwvlx7suX77UXn31lYAB4G3CoLVQ22ctZLBoZaPHN5SveM+a6Kt1l5RVe1/Nli6lvFfQurPmZSbC5xgxilF34CmrAV0enemrCXhZsE7V2hvyiqD/aooP9whyK+yDWbSJpD366B/s7nt+qGgBh0LIf+FFF3o6orDa07CFwoznrgCkC3xG1hbmZ6xRcafE/TJOBoWVQamNgOmYXXftjUL2yaupS6tslO2wo4/9iiRtOSORLgu7bHx8XPtGHPcAlnluD+rskR4YgqRZG6RSOT0v31tpS/zoutP0xHWKQ7VOmyBMPI8oq48/SFilVG43F7NIGkhNrYr2JkTWVOf0dii+D9sp6i3zQDSqEgHrvC+oUFRr2dxC1X7y40esWk04Yi3yPCFVy17/hl3tfe87WA9d6KqEV6HI9Vg6l9UNUg4CyYtJPIsDQV2zS8slhV8s1rHHneyT0TNJhTHXXHOdX0NonueAsHj851I7XjZotpLKQ0UwVygPcJBRzy8US01xD/kQy6cWuJCLcX/R+6YgNwSryibyzQkguC3MjkCPb0Lvc63VaMfjetzjduTz4rR+85uX2+io0+94/eeOOMLecsD+Mn7xMPtu3/ZvnmE8uJVq0cZHtqgDa82Va21yqiCvdPSxR1tPX6/kQjl8REwYLs05azo7jY3mU/x8OgCRi9ZfIuRueGK4qrpk3YXLBZIlUzrAgGQ8b9YYY4j353mR/ij6C/OdQKNBnXm9lESCogp1eQ4uho9n7FGiYyUut+vo8f0//In94pe/DtMinGNww403WKm4IGE9ACmuNYoDaO01+QJJ26rVSs5LJoxm5pK8ovp6MTglu/ZbN1pWoXnQA6vV7BOfPFy5LXVfnS9IS7wnTADx1h3gigYpEjA8vHf6J9zmeLAdJA2i6D/81knbBNFbXjNTzlKtiazvVoa6GjWlpC3Mz7fRZiycgw5Nq4fWJiXRKbR0nUYoRJnp9Wj+hG4QaQdlUQsoaaI7N481ee655+yfL4xatZ7UhqEvMiJrR5/wFRXHKahTKlWfpoj+PCSGNBesu7dHh8sHOIdZP5aw/r4+bRYOwKc++XmrI8Kd8qL5TTfdFBbc5wBB/YtKA3h9X1lQR5hAgdlS9fxTOUk6pfyGdYNcHz2OvEoYiAaY52UD6rEgvY4WIs7m5Y5Y4nEv497ZzSgally3jEmt5DlzKmX9fUOSaHnqqafse7ffpWfDfwe881126KcO176OdNNISfWb8UNMGAioRJfQxNiIjW3dYt/97l02O1dUnffiSy9VZ4/wCKaz5/PKAbu62JxJ/RvyC+5ZXOq+PkVnkDMkSBBCZ1B5rrcQFDK4K6UjQbxBjQW0iBKtTU2FpoqEDQ0O2uT4RDst6+/vtSnVT71dDwNOvk00ghGgzZBGh8hdJtyV5yIlq1TtqquusY1btjgwxXiXzk67+OKL5QyY1xv7XKVlVnP6Y2fe97eoljVaKoOkU0itYh5//w9/ZOvXb3ZkO6DW+a6sfemLX7Levm7tEcn9CE12MM0bKraNo+G5eoupH9QIAkr5cTuGYvx54t6rT1So7EOjfAHFvcz5MGtHvJj76pYB3Vt+zmHmAfBhqqSQPwmZTSuUxDrr9UFMjAWkQO+slIoOC2WGnm7mzXpozWu+e+u9VqxQLvIcG5Qaa330cUdaR44aoHsyPodwiNwTj0sNjIkEg4OUn6DN+dgJXouxIc/m67zzLrBn//GKroND/oMf/EDXIoApCJe7JU0qf5a1C6oDHFxnS7EYgSBOe5tANi8NcB9x3WL+F8svbsx8IoTYVCHfUXmMhxoeGmkKX3pg8pQujIekajy4IMmICuB9Vp9LyOcHvX/xMvvG+ef67wcOefTwsV4vDrCZjY2N6v0mx7aIVLB27Y1Wrbm863nnn2/1pkcVsSdWWEgKI0uI1yHWFsZbpUTyQ6YFhFDYm098IBpeyimOHp6LeBGUMMnbMAYYAg4/h1czk8MIEQ938eaO+rqQvKOrGhpGDbhSUV1YDKka2ljz4qjznnGvnHLy6TZD6EnbZSplb/zXN9rhHz9cCPb8grdoclgKc3PtqQmkPzwbPc+sWq30rJUDlwDQEAJs2IUXXaLuNEeJHbR898H/x/bYYw/dWxh0IgfmIvnOVch1ODqtMlgoHUXHyWeKeRV42yoTxUkW4AA/vv40HVwv1nuNy7WCUGrfNjdIag4wi/CaGmhNw3E1CHr7DF2Va5Ipm5mb1aLNzc956EKY1dfbbufiQM3OM8LBgSRR/SgJ1Gr26ONP2LoNE1YLTfuiM5rZ/ge91d75rrcp+S9XFrRZevv6pWkVwwfCiojETk5O2tDQsCiOcDCx+Ljq559/xdZec5OzojJpO/PMM+0t+71V5QG1DYa8kzXx8ZGOMjt44iwf3q9dZhHAFLS6aPRG/IyJ8YwuDeTzapm82FvL0uHgAn6p40gHFAzUmzH0uRTbA9E/Ug3lNYPkKb9TZJJ809Uy2ZTcj9Q3Mx122dVX/X/qqzwvv+4QliXJp3P2wgsvyivNTI/bKy+9YNde+23xfTvyHXbOOeeoIcKHbfuoTJ4/B5c/RdmbR6DAPB1ijnC1IoMtFDuUv8AHCGWjvE3M310s1nNwiBaRaIBnivxdZiupdVIhposbaFIC/HKh0i6orxnFjYbKiKw/xgQnETuv4CMce+wJqihoHEjC7Jijj7HXv/71Mi5TM5MiXajxo8kAbHdUHNyobKIeayKnYtkG+7q0z0g5Nm3YaDffdIt15XtEBfY6f8OOO/5oH5fZpPfcjS+/42lZMHA5Fw2IXnR7YEoOY7upltsaDvyeEw/edLom0vNUeWgcRh5SpeYgFDdBmMvq4WFBxxYtWuzspECtw1I6WuZeyEsk3iBeXPDal8acNCBtw/0sW6HoPGIvMZS0gbjQdes22q9+80erUKZrJKxKY4JCtqyddfbp4tmqnzPwgBl1QdM1G4LWv4hww+jRjfO5INQoBtYrNj251c48a41VkNbs6LB3vvOd9uUvf8XQ5/Vaczg8gWYXrSHXuD3yF/NgSjryyGqccEK7AJVAT8N7VGtlARNqzIfJJaCFHCq0SsqaekikyQZi67hahg+q8rAX/EejOgFkJsfFn8XSX3zJFTY5MacOFkpGV1x7jVNRG4HrGmYUsWEIDZkRBELK88Iw8iypp6+5/Ep91g477GBHHXWUJGzdw2+n0ZzyziYMrufeNevr7bPxsTGV2DD6TlsMwFU6LU/IYRG4Qm0fWVUiGiKikJrJE0lTmbZMP+jkgLCylENnsoqaRke3yijy3FnnOC4Go8rokZg/I2DOvlAE0NVjR3/tWCvXvO2U91t9weq24By1e4wCXABq3KJqUnopLrSbIsQ6C5GKxuWEkPu2m79rr7zySpjc58+PMtOb3vpmr90DPtW3lfboN+ZecSzsUV5DM76GnGsfeVeUkzRcjCDiIE4KImopWuL+605qyVITIlc4wB5+IE7FQxMTRU3AziJxJoeLo8F44cN5KpAG+IBY4lHZgf7SojcnYzUV3nZ1e100gF8R/QVM8k00bb/89eM2OVmU/AudFa47lLCvf/2rQoMXL17i0wPZiEHrSXlXl4NTkZjNdYs5E8oWE+OjlmiV7fgTzrPZYkWh3YqVK+3yy9dYPhgO0Go+j+ti80Rks81cCSFLLF+ogyhI18a/c4oBkCJ3mZqsE8QJieGvIHRmVik6F9WNg3teR/C15GFwtkdBrpTh4SEHpjA5ZoXCjOqkd/3gR/bM35730Y8dWVtz7dWqxQauR2CseY0TA7l5yyZdmyRiBC6lbMvIiJ1z9rm6nje/6c32mc99Wt6Wnmc2itrN1CEWdLe0zgyy8kFvhbl5eV5+Z5aQlAMS5hypw6bsbCOMuLxlC0ZVT7uvNYJlvb39CpkRoQMzYM9QNqJ8hJGP4evGTRt1L+wnNbS0kK/13LFWQ9cpTuZzreKTTjpNooJcE597+RWXK0KQqkqomqhvJmA1Cl0hFgklJyWpKIoU040DVfcG+gvPv7Dd8+zD3lp21tlnW61eUkO/UPXgiSXXm9vGw+bCnJddUelRxqMEv6Gse4vpHPfP+/I92HqS8OXgikwgAGTbgOGFEghdWtaNeqF7gzC+IsD09FjyPW6I8gcfIP1gkcC9JQtJDh2AVktkdulM0UDd06XEH2OANSNfZWP193XZ1ol5+973fmKNZlKhK3U8NvPb/+1Ae+97D1Z+Se6LkvzwomF5D8Lazi7E3wBSumTxBdhElhIGoNaw8bF1du21t9vLG0cEbpEL3XHn92V82FyQDWKtDKOkDp3Q3xqNAmsRv+dKBXHiA43mDsqR15Jrce+cVh/9gZcFkeTjIBP4a7f/UggehMBleDRMzZUXiDrY9KxHvUg7Hn20DXvyL0/Zzx76jU8jTCbsyuuu0WhG16JzBQ82iCis1rLR0RF1WLGpyDG5TzbELbd8x1566WV52z332sNJFqE7is+ltkzTARsIYFEU1nCARfsLJSnm6cxMz6jDSnsmIs0IDII0Q/VUzXSb8kXctF5OyQqrcKTXpWR4koThfM+F45taX4BBPCvOQWmR69/rWlj70dExYzby6aef5dzwTEYp2iWXXqIDzz1KDxt1RdRJAoCqSCPhz1CrGDANX1GR/Oyf//yn3XH7nQFdb4gAc9BBB9p73vs+9TsQusOum5mdFEMs18mUQq84COOobxsMxxwnDBtGZXZuWpEb9yiFytDMT5sga4G4ROK+a7/egg/LFHHGR5JtoVAfmRxYd+QwY60MaJsF5IHHflz1m2qaHdaxYLWq53wc/GLVxc548EPDfSqao+bAgsVNUw6EAKkVZDI2OTlmjzz0R5ukKRwVgjINED4I6tRTT7RMh3t9lpB8EkOhnKNMWO9KGfkcxsQROlngUFeemZqwf/zjH3b7nQ/pCWNxb7zlZlk8MYkq9PXStVIVuX94eJErFtJ+RoknoIYxD8UgicqoRnifL0w/L8DN+vXrbeXKVQrTOejRIkdiS7nITFW/Rr54QP+vr1hHJ4SOh4nWwnq1ZPNTkzY9O21rr7pRJTJSiHPOP88Glixus4TwjKqpJh0sRI2QL+RKSQ8Iy7xs41QPDvj8/KyuDSOxZcsWb1ur1cMECBo9OmxuZla5JPeve04mnSSQg7nkHjWi5uSbEYQkdfGKgHsvohzWGw+4aHhYQgaEuqC4eN9tRtIUzipCCaCh6K40uLfQiMrLGUgFZWbWZqenlbsiLnDp5Vdp/TE2O6xcYcccf4wNiIo532a+8XzVNBIQfcpSNIggqgciiYpHviNnKIqyRtdde63WRg30zLhNJ2z1Bed7ZCVpHs9rOzOpNiLeaFRUfyZlIn/m7BD5lCrwsL3pIIUogbrfaO10FUhPZcNgbdoh773may1kPVAz8J7clEZNxB5QNsLkxIQWQECFKGVu+fk3C47FG59gqpmLuUHL48Hye9mgesfGIQfjcJJPefzuvFVChsmpKbXcMT0PdtE/nltnf3jyRc/VJHHqXucbZ52qh04k4DfX8sZ3NHXzOYXGW0e3Wi4LTxWqGGULF+vmYJYKBdsystmuWPtd1+LNZOzk00+xHVfsqFCPh8XCc10+bNlVPQh7hDzmaS30NrG4+QgV3Qv77BuF6qLRhQl2otlRH/ZZw95p5MoQymuCp/p/HVwPkx34wxGLoMEkvZq3zJWYElev2PnnX2a1io/M/MrXj7J93rBv8A0eDbDRoM2Nbh3VJEM+n4MLM8nbEL0VL/KNyad5VuSQk5MTPi1AFEpU9f3QdeUcDebvHCg8Fp+FJhKbkL3BgSeagxQzsmVE/160aFjPTCgw6RiIrAAwNI45wI6qE45u4+9iULy0xF7kOvEu1H5h3oEjMEYGQy55n9k5Ic3c49jYhN1wI8BbS4DboYcdZu/6D8Ta6GiiH9mbHdgLVDk4/D5NsiXPWpFcqzcTSKY3mRIwdd655wZCBAe+Zbvttbt95jOfFV4SU0D2yuT4mEvXUtJr1dWbrJp81gk/XoYEvHTtZv5kHbmvPM00AsYoU7oaqgz5fdce3apX2YQOJiCVUqnA8vDGZRY9AjAiRouQ4P1Er9ltd3v22We1+IRo/NxHS2QUIgA+8KV8L5HQgnR1d8nqR42dWMfDUqthvcoGX1BR++f/86TNFH0qu4crZq993Z526Mc+JiaJM6a8zolECRuPmySkW7J4sZeCFhyBFpCBNW2YpDAvu+JGWyj5Qn3ui5+3fV73Wh20vqDsEPNNrpP37+sbCF1CPk6D+/OSmDPLsKw8rBhKcai2jXJxkoI2YzikGAQYVarnBn3l+Of2xImItup16FYHWRzJ6lTKNj81pbEjay7/ltISNjVTDd79/ve2ZUw5zaw76wi4SJ2WNQEg8Sl+LlPD57Ou7im8UcA9QkXAIsaRkJpwm3vtyQMgEa35v2OpCnCKr8iv5fDDQIu1Sjaz571QZXkGPsRtYKDfe52Z3IixTXroyL1jGOJzlKEALESSNwBhQvxDnoih3mWnne2Vl1+W89i6dcxuv+MH6osmGrhszRrr6e/RffAsqQGr8yxwChRthV5q+MVk8gulgiKABsL1Xd32x8f/YD+6//5w/z6U+yz1L3fI+C9avNjxFgFoqGEWpN6CAin16VU7rLD5BW/KUDtoEBfUtI06Rtlr7ZhKjKaMYI/PupJ0zU+/fVqLmTBC4zro2ofHm9GAXt+I7iHYTKB6tGjRihfDHq/jegmJw+FcXuaUer21p2dAi6y2LRYGLeHAuGEzqCVLdL6WzRfmlQ9pYnqrYX944in7x/OjVmEqedpJHb293XbBxav13rOzMyK/C2TBK1a8yM2GIQTiMEUDgbVmU8c69Y03f8f+/txLlkx32P4HHmAHH/xu6+vvs54e96gYEl7L7/tA5pLrUwk1RioFQgnSn46eR+oaD2J7RJjr4Z7UtRIQ4TYVUt4UL+JhlXtfD4vcUIX+YCHLXprzdjYyE1oXG1YpFG12YtQe/MmD9qcnn1MueOA73m6f+txnFa65IcFD08XE8KtuMb1UzlmAwMBByYikQgcMz5CwlvQoKkZoh6UAACAASURBVC+SEkH/43rk+UM+SwgevRVejnyT/LEdjaj5o+agWda7feTFa1V58mjlWGO8L0aDOinhdyy38QxUMgztlLCgBKRqaDrcX+ezc5iV1kGlRXJWhq0ksPPvf3/OfvzAz6SAggG54OKLFFarYSD0BUtqKDSTKELo6ZH+tkcTC97ZQ5MDnq9ldv31N0qQn3Sq0qzbrnvsbh865FBbvGiRX7uqIR5xcT/cg6JUzUT26M3vAyVRE/9a1Ev0pQuz7dIqpU8MF3ltR2hukOe984pjxJwCmMp15W1gcFjaQXNsiNlZhTaEJdwIFgO9IW3UgBiSvHMBXJwslTZnXQ/K8ycHCbBmsLG4CBZLeWgexYox65E19noobJxicd7ynTnbsHGTPfAQM4MIq50yxvuffd43dD0YCRYAz0EzOGmvqHVwWRcKMjQAV4AvhOdszrkANjz6+B/tvvsfVqQxvHSRnXbqqaK+8X5sBJUGRM9DVBxpWK83O83PhdnxRHikeGij4oFCaU2x94ZorCehspPMPeRct26dyi4R8nedLydH+rQ/jzAUVYjh4oSKgLuAWklxEw8wsXWL/f3pv9kdd93vSoL/8i92/MknesN7kkhnQSUdWE0YEAyOG2gOoYumYzGGBwd0aPk5fFueLZ8PgwyDhSdRKae9ocu2bNkyeXEOH69nraenprVmPGcOJNEFBkM0UhH3TfuBCfQYWW/hc2mdhbl5pV4idiDVO+PyLjxfZv8op+WAhusA12ChlE8H3jKLRW7KYRgfH7UHH3zYnnn2eWu0UgK9zr/oQoGp0VBCc/Qw3eWLMKZCxRnNku+y6ZlJIcystcA45FcvXRP6fVMqWR59/LG2eNlynR2+aPTwqMCxE0Jw1aMR7gspBevhDqDiUxOC6gc1a0lEaY4VHG+X9eV3wZCkvf3zOy9poWTAg+zuZS4M9bmqjY2O2+v33VcbbOmSZWHkxBIdZh5Q9DRelHdVAw5jLJ+4En/C6kb4hYQHC+IFfTFjas5jjTKm8sLE9QxXatRsfnbGCsVZe/yPz9qLL48GnVk6+ZK2/4FvtcMOO0xIHTKX6EvR4UHIw0bFiMzMTNnwokUKUdTMQFRAaJdyZHWusGBnnEljdcv+5fX72Be+8Dnr7emVdQUQEQIMUt2ZVyTA1D02NS10WOfIueWQIsWC9RaIIhX9jIwGQEcElraFwV5bFaQfDmhUN9jmdd3jKpwObYV6n6DOoVxTSKvXhefmpm39Sy/ZFWvWqmtqaOliu+iSS7xnNXhcnDYGLl63No8+wxs3+OyB3h5dGznm1hFyYZPR5sACsoEroBtNWI3UC903ArDKJeWwXsP3ZnCF0t09WnvYSbGOT2TE+5B78j0+FwPGSBNQaLI+RNWef/55HUZVPIJUjdaX0D6R1IHGEHPgqDDgxeLEB7w5DqBaKdmG9evUPLFhEyyxhO3xmtfYV486UjVxDDPPyidUeHSj/aJ2vZR1hjY79gRccgTvuL+nnnzSHv39Y1p9bB4O7+TTT9VQcVoNcXC0xHqjjosvSISePxs1vQfeevkOy329lf54aZCcXcYyGCcL9EvO0sycI+g4ocTd153WciZMTioKkCLwZIRBLKZD1ynp5bJBPY91hDDX0eVNBrS4gSTyPbwNYWtot+vu69Wh4X1HxyfaKhiUYQiZgMyxfj29PbJWqO17aapm83MTesB33/ubdkkEz8WDP/e8sx1NTPiB4XdYJEI1RlosX7bMNm7aJMALhQi+6MFkqgB/0lj99NPP6KDv+/rX+USDLMp83TY3O6frrahTo0fhEfTHWAYiJ+MACGCq1rVhooavuocqVX2PA+8lrj43dIEhFi09axQNnyPOHh6367ihruu58fajM32TRaQREGdkdL2dc/aFyqcGh4bs4osusmTG5yU5m6elzc51xQYB9cuqVu2gGpxh8AeBlJq106VNRWkHz8i6cj/i0Qq0c7I94anWX3IwKRkCn0CfkaFns4k1FFBrDvusWuW8g4fmj5WrVskQ4+mXLl2qw6Mp8Gzmri5J0PL+XpGAI0AImbGZkJ+yRgpLg+wMnHPC6S2b19uN199ko+Mzlkhl7OD3HGyHfvRQa9B2SQlIE/e2TWpk34lKSQoHSYTcWuW9ps3NzOi6rrvmW5JaUqkrmbQTTjzB+iBTwGnPgrJ7js6e4F5UbQpG2IFCJvwBotV0b6Nbt8pB8Jooy6soJCDnRDviXTcaqm+zfomf3HZhi2Qez4GahLOjGCkYpu9Rv2V8paBqs6VLlkpAm79X6VlVztohDwOXVA3QeLS5eW3KVTvvpA8Tb7fpJQJCy9l5FDOcUCA9KknB+phFrCULB3+22Sjb9+96yCamPETnogFaPvXJTyjsmZqdbOfXbChH/5LqDIphFtgWjfcMOKZvk02KMr7LdHpLIA/He3H53S73sl09CsM4sPCvuW5a77zX1GF8BmMBiBFCDQzQ5gVwBed2Wn+Xoh8i2v39MkwAMOqL1ZDqzYoKVNjaLjzmgQlIUwdbrBNvk+l0rnGYsEhIXuf6ynbiCSfrcLEZ1q5lHMm2nmoZHTMBdzFiYB0kM9rtE+5A7oiGqNFiMCmXsN4ukOdi9BxoSmSvrntV9FMOD9dDvsyBJ58FB/EWNG86YJPyPKge8EyEnNar+j4HkfQrln2oZvh11drlJF27DrDLFMWUjIOe0cR5fx4R6FODA9GeiB5NO/HkkzTzN9PRYUcdeaTttNNO1tPX3R4Y7kqOrrAiyaTApKKGzhfrRUhOjXfzpk1215136TPpu013dtipp51m3QFJFkmkUhZar30TniPfJ3Xk2jXcjH+Des95rZ9zgKFiD3leDUCFk4K1GAbOC/Nwud3EA3dcJsojJxpuKDeAu0cWJOorp3KO+gmc0OCshHR1N27a0EZVyXFiWURsF3ltzyPwOIrnO+kzdI1eNTGEw0CeGRHJUpEDX7Mli4Zt84YRm5vdauOTs3bvvT9tP5xyuWp7772nHfaxw6ze9HoX/7FZCMuY4aoQE5YLigK1mnIxQDVm4fJvroNNBljGgWKxObBYOsIn1mNqhnqnayBJlLVWdyudzcmy4528tIO0aFZIdjx05Hnx4OKxly9f7p0mvB8Qf6BJ4pkIaeOsIG0+SeU43zcizK7cEL2ue1yMppfEvM3x0ssusWee/psNDw3bBRdeoNEVPDM3TOT/EPKZ7+O90GwqNjk/5PPTGTSavEykdchkbNPGTWp/5N7F2ir7xDoaBRSoi+hPf+yCDCoblmdPuqJul1Dj5hoAHbkeqJSF+TmRX1DHEPIaJkIQwRA5DQ8NCXhcvwH5UydOyFtlMup5Rs2T0JW1wuMT9vLzKOYAAozXQ9HigQcfsod+9ogM2qXf/KbLBNHvHO5ftfgwHV5chihC13R2mdawUbPpiUn79a9/bU//9W86H6z7hz9+qO3z2n3UZonDmhifCCG+r4sojxIYNI8GUQOhsSaodWjPMsKFXJq6c9DOis8+8ptFxAjMN13T3TevbmGtWCQW2vOJpoYUUfei5zXWkLiQqMHEQYSooIG+hK+0e6E5FVrAfMM0BSpA8BfPMnRBKLw2J4uzkbwe6nImWFAWESs0PTlhhblZK5Xm7bbb7rZKVfibVSo+OOsb3zhFdDwOaxQJw5qh37NkyVJHYTmkUTS7s9PDopBfOs3QD4NvXJ8WoMHeoS2O16vUoc4npEUyolYuFLGq3eoBFlraiSbTVtt9993VZM3G5UHwXhxOQs04yYADDW1TTRvULSs++TxeBwupxoXwwD1UJix1EXGiCnFnw5BoQDmMAtfOPbMx5a3D+BR+l++DTQCm0c5HLZV1Fxm/XcpquTHNuNfAC3JPIKWkHfybe6F5RCWJhBNhAFjEpAp1fg4kkQLrRkjLwfJIzCVvMBpEVj4LykeaqM85iBQqrcFwpJl052QYPoP8j+hN0R1zkZnDCzc6TLHHywoQE6vLa+UxR/aupAFhHOL6Jj2i9CgO0NEb1ON+EFspUHxZ73Jx3sZHJ+y7tzDNsKa1xSmccc5ZTv1U77VfZ+TCtWceg8oXCsr52UfqE9cUBFck4SC7Z3eBAHJ9DjYRC5x+rivyHhwHSVjiobvWtBgx6Vxkkmum0TWtkWhaZ65blpzFcGU/V8b3oUyIwvnsl7gQ0VuACBLqxFY9vPHM9LQsBt6GUDbb6eUUwh82EhcDOIQV5RB70/SCWtnoQnns8T/ZY394UkbEZ+Sm7MijjrDBoX4hdlh5HpZ6cxeg5rkFhjiBtYttW5EYTwjiuV9TVpVwn993BL03jNx0obFYp4RiSU9qXz96TS3lwrvtsbcOHR5WZZX+Pv2dz8SzsSasnTwmn1XzLpdVK1c6zTJwwHmAnuN67qoHRT4emGF8H91o7pPnAT4FRsD6z0xPel4ZIifPxXXc9Z6RfgrggVHEuCl/DZJDft39ogyKg02ZLvT9ToyPO5NIw5l9jIlyZJWTvJbKs2PzQaLh/VkDMaVk/NEYg0SQtgWV6FwelYMbc9Kx0VE5Dg6gpjdQmhTYWdckO3jU3DMeSyIMoP5SHWFmL9ex4OXHUGbhPRj+xvvEBhb2AmBoVJFgrahJO4EIMNJJ/eyL2C+LjpYbcP6vZi88/7L94Pt3qwIDR/6d//7vUgrxBhQOPVx+LyG5fDBytB5NxsgEOi1ALfsUI8nzi62ArHPkLHjakdbBxYjLS4f2V3ETCJVFPVOZxiVDlDMglVEs29DwYhvoHxRQ5cBEXhuG36EkRElk8eJFNiutWQcmWGSsI9aHkEYxOpZNbW8UkskvPPTBU+G1hUiHkYtxRg5Op1YuStFw3boNdv0Nt/iUd7G8Grb33rvbRz7yIb2/K/y5BUces1Aq6SG47AfKBt7xoQNLaBg6PVgMrtfRPY82+LtI5gAUoJa8V2fegZaBfk2B33XX3RQ2Tk3PCQySqBh0R4TGOjoEtmGQeChqN6tV1UWjqXP5vELNZ/72jHKZAw84UPegUDp4WylKkJMuLOi9d9xhB3l6CWnLmHhxHw9EM3zMg2K5iAcvFYlgnOJ98dxceSSmF5R+fKbt1PSEDrBqp8H7gETHLi5ycn4WW+AmJpiRO+RhNyywUKfGQzt1Mi0j6sQJBqF7PzHOAQQboIe1IqfdsGGD6I6sNXk/e2l+jqnvPhGANaDUFBsTiB4wPvGQz8/OKn9nXQX8BPJDYX7WwUPCZnAJOtF6eqwz12VbtgC+dqiZgc/j4PBzR++JLd248FVr1tTNdc7Z51kuS9NMwk77xhmWD2NGNGm+XlW6QN6q2Ukq73hzSCz7EYGgPY3zIv/n/tgPrFVspMfAqhRJpBRok3HvRr584kffu6yl0EXuOKML5hdgTnnu0KlGcw+38AqxgIzndC4mm4nQNr4P1mjRcCjF0PkfSNKx3snDQic5ItSEztyItxB6Us8NYZHYaAAuszMT9thjf7Bnnn4xdNI0RXE85fQTdYB4LxElFD7lrVh2Jg8v5nuIgvHwo1wOOTq1Xg8LfTQGm4tQ0nMl18OKXi+WTJRnZbPW09tnS5cst3Taa71bR0asp5/m7U5xlMmXyWy4Hx18wLLpGUH66vrIeWSAl1g0vEQlBUJRSQBpyIELsRNBM+aRtePhY4Q44MuXLW+XimZmp2XdOS3IikbVB5rGly1dai+++FJIKZhQx3QDrw1ivHRdMzNyy0ReAuXI18TbriospguM73GIQUmdUFO3gaFh27R5cyj7lLUPCGPj3CCfUuDaWy6iwExbryQAYIk1lUqqbs+9EplheOMeoPWPgyDEP5AyOEQYNcJhSRmFEk4k4uAE5DWpPde2TUXwkR5uuB3xzqkzCU8moCkSPJQmecSDSotmBYEnbBedUY3AmOy7776qj8f97Q0S6GA5b53rJudXX3Ag17A/XEklODmGdisF9W4wIpioxhFHjjhD0NMYnAlGIfGTO9fo4HJx3d1O78NS7LXn3vb8Cy/oge6wYpVYSngvXudzQJFc8Q6N+MEsLl/Qvcjv1LIU3o/F4CZk9aQ36zqxWCfek4VAw9fbmpyxFRX7CbXGx7bahvXr7ft3/lAaQlEB4evHHBXC4G7p82DRmE5OO5rCRw3faijnJcSL4SgbSXB+AHxY8CgSzsPn2tuatlGdMqh3gE4K/at5SEoIjbUXEIaIdtWjDv6LFpjPldxL0eVNRbHLddjmzVukErF8xY7aLNpMKEKE+jDX5F7B0Wz+zXpxSLhHDgossfiFCke0ypk0RsjRejYGUYd714ZyWIw1hjmG2Zo+MDCgtIEDTJjHsxDxXjUNJgV4OZDfLWqcqOsBA0Byb3wW6ChGgGtWjZRDgAcNhA48KgPbuA+tSSibOTjjmtwcYkTiXL+Mg+sbXDgAZSd1yczLK0rOt97QgQc3wdBzTzDhRIhI+GxaB5kQ6+/TKBLXE4tSMj6GlahQTkpcdMLcbc0RGB7Wjb0TcQOF0YFJxnPaHvCKZdLI6WfdYq3Pwc1SEJh3iSYdSPjQ0qqecVVNgW7cs5f0MEhCzR+860qhyiwKibv3vjKR28EPFp2DouFJRW9aj83vxP3KS4JiIIuANaSlTAJe0tXJtlvwonypfr/sdVEOKEgvB3ZoyBuL8XYuadKlG2GTzk5PaF7tj3/0sG3ZPBbqmGY777arfeLwwxXaU0cjFOfArVy5wjZsWK9Nz6FsAzZBYDqCZzzVqE9E2KoNWSyqiM5hZD0wHJLHIT+kuVoHOWGLFy1ViyH5Oxt+enZGeTqenPVkU4Im8wBZDyHdDdMDIb9y8GdE2lE77bqL6nkCVBLu1UFcIyuJa8IgRuSe94ujKXffbTd75dVX9bO48dXAX3HJVw4qa07aIo5w1TefRlqG8TNCzK0lMgThN0Z03br1Xr5iHAeT6oLgQQxdKzUIFA44Ue7ivdjYTmllH/kAa/YQeABGZK+99lLoSu1206bNttPOOwmEZG3Gx0Z10GNr5NLFi9spSFdPj6IRIhUiQYnei/bqbYkC7wK6z3uLRgn9NnQPRa9KAz7eGULN7KzvUT+8pAwdGvki2iRRaMajnGiQKOdg/FlDdSjh7cVDQD+cUlVJRhtjvXnzqK1cuTJQOSHpIEAxrOuNnykuROhVdnEAxoQ6YwyHE3W7uGfSCowv16gJgb+8/4YW4QCHgxonb4Rbh7/sOkD9No/anEYzFGzVyh1tdsZnp9CRwYIhrk1xmvchNCMEpMYWSQexw2Nqerpd3iCfYXH4fTY+D165cbeTGTAQgDx4CGiKauFutmzdulftttvucBCnRY9qhx1/8klqII+80wjD8x4Io0dubkQ9IwiBd+MhRBTVhejo/3UpUg1xDjNq2HRxTi6bVSGX6tg+uY3rQL9Xqn/kcINDAmswALxGiGc2o8OD1+JgIYvD/XPoXrvPaxXV8FpFMEGtYnJqQvcVw2hCcA4HXVQ8bCw4+S/q+9G74X0U7klQzdVFuKb43soP83ldM3+PKUZPb5cT+pFuEartSK84y4FPrWpCt0/Ac8wjpDZdcNgn9Yzo2WXTxUPFvbJxd911dxuiHFepSO+K+q16W2HepQEG5wOg6e2RFP4j7ZG1IzReuWKlHAHvzT6VMlGYmAgOgdGMaDH/pv6u2VdxhCXRkLrbnCQSw1KtF+iwaKeek1Ka4nDJmAZhAO4PcIn8Wg6ICEo9x3hoz42JbMi11WJIWhiINxxMqix8eQTgiDZRCgdWbYQouYSxrDHXJvVRjblU0rlQBPXgXWs17JEfMmaDw0bdjgiSjckCLlqyRHmbtGeDcgULNzDg4SgL19MFAr0tN+OwKZfr7DSQSQ1SCiUPLG5nR05yJ5ETDMghS5JMS5+KjQ4QRrsgpG7lK3i+uXm77rrrbXYWhUGsedIOPfzjEvCW6DYHIoxu8PCfMNbHo/BweN+h4WFZbLeqHpoJYg9av5QuhCAX5uW9o6aUPGYYQA1pgXo03hgQig0/NDiszxCPWTNnMj5oOekcWWp47Y3AxMICD6JPv0+3kbScQyfPyJYtHq6LMeRDwvldlRSE+Pq/QUoxMG394qBqyIPm9zTLdnBQFhsSjUJfGSMvufAesSTV1+dT5CIUHRlw7A1KGD5Hx6fIybsDGs3O2dDwkM3NOrWU9+rp7fayYhN5Xu8K4lDw+0QNdOzgtdk7pA2sobqOJNnje5D1YCPLcBRLEmEgyuAZq2MLKSBCaqiFAQvBAPMzyCGUsYh+hhYt0s+5T/SkWb84PsSBwKbjECE9QpdK3lsaXdt0sajju2SS66ppRE44fHymIkzhDN4pxl5irSgDqsOuCX3WAau4jvw75tMKuSW4j8P0hvnwIByFl0H3MTgY5sRDP7i6hfWQNEkYzSE91xQ1NBdmLgdVR8KJHMoSaBgpHNqmESw1Wak0kB/5IKyYL0dPR/4QifiIzmFR2ORYEc89E6Ii8n3AF7yTwnb6GFWg9+6O9es22g033KiDy3Xstuce9qFDPqJDyesxJEIc1e/bLdYLv4vnhfmF5cMo4AWwum4pPWRSGCMFyW41PwvoYWg2k+rVweG9sRGaj3kb90hfaewI0XCpICbg1txRXB7qDkxKn5wUQo4n5GHKC4f6Kd7HqY88yEIbrYWUwOt5ba1GiOraw2xijMhee+8VaIJ0L3W258KqZS6Q3rlu5U9C3D2EjnnqwoJ3VLHhhgcHReoXaJn0/JTckL9v2rxJhwKjBm7B8xobnQhlvLyaNYi4IjhFXVec5Q5+5iAi98hhxejwM0UGAJzq06WcBxMqKfaW5GOQPgpD1+ANq8QVOMbq2qrVbXxivL1vqFZgOGhIUCkmcAqkpIEqxbR3v3H/S5a6QDkHgrlUQoMVBi+0CUYQhiKRBWejkmkcQK7JGa61jcHnekhz+LmrdlAtIAXyPNq7rIhgQZgH5ElVsgyCfP5zb1mNgC5nkjIlLlZ740d3rRWtQ+1wuS7beeedVfoZWjSsXIcL2mGH5QGE8lYpYnh1uaBYqLEPxOqeF7CAeEM+VCFVyXMCHfSG10yxtj5P1DWN8N5sNDYNrB/EswA7IDJQVuGiG1JzNL0nr6c7o1Bgoh+AQtbO+MYZIrqLtSUVDpBP71DR4jFZjsgAiRwAjyCu7rQ838hCtfPdCpVFZEDnCKUHmrYVevqBEmAQh35r4rlHJhIfQENYAu2ICvjDVWjOjJsGEj3eVifBsKAjrNqpwAlv0GdTC6lX3ZgGBxcOJ8Tj/nzQ1oz+zfswo5XrwZsJIBGxH86413H5TIgo5HYoNsS8LZZ9eE3cILxvDKnVgkcXF/cS7hFjEUE/nAI1WIwk1xvzY1InDoL6o1MeNRBOUm9n40oNEo9a8vk/UeKHtcX78W/xAIICKN+X5GqvixJiANmv/eIf0KGVs+npMBKF0SYFat2wAEuaOhDJPSDYqslLnZS+VkaXIL/TbHPlNYw9MLCoHEiONVQSeD93DC6JxLPCeVHFYE3c+Xj/bDrp2loe+XjXlzqFqLA0mzJSNLrwjIXgy3i7cCLVEkWPqFVmaOlzuVmBjkEuKvHLB2+R4A6bhXsBIMITkRuwkVhIwjLfbJ1SAwC5w7tJTKtUbBPzuSlp4LYSYhXFRgNyMg5k9KocRAe1PJ/i4rE6nrT78CbAEfIVvg/ZgfIU3tNDu5r97OGf22//91HrQHIllbArrrxKVpmNKzkSych4aB05tHgnrCpGBoOiujGjKygvhEK3y6Z6mYTP8oVPKa9nLbztzj0714HCh4d4zmwSQ4YGAwmm+b1E7xb7TGMvLNeJ9Wajq1QRuLh4FvIcrsU3LTK3PodJXNhSSd4KY8drXQYXxpnTL32WLlGE58saZyn03NUjMURisqWZBtEVpIjmJEbA+hMBqbc1tEy64FnSmXIqw3h+jXAbeSnXHUdv8nPqvoTD3mTviv+xOYBoTTKooUnC8zwP+1U7DyguOTTeFnIPa+NtkhhJclTPodk33BBRCOg6ObaDe3QU1WS8aN8B5+AzyIcxBtKRAmkuV6T0GLEWFhjPiuHmnoeGFjkmQVQSJivKgIeZPy5BhFekf91VXSI4mWx5muYgYsL7xoOqpXdlIcjrdWM8qWYFB/4An+FVAxp0vOEj7jHuT/nxQ/ddL7E4z0e7xOkdGxu3WsOJ2yIwQE0MdDo+Tq9PJsRo0thCrAxhRo55sj4NnA3FwWEB8b54Bw4zG4mDy8YUZznr8iLcdERteS/4qBw0DozXZZ0YEnPVjRs326233i7k9JjjjrVddtlVjeNC5BAOr1fbmyl2qAA++ThFZ1nxYGP5ieuIvN/22Azau4LeMg8ecA1LiYohm5V71EYMetLx4Ea1CZVUAuvMx3e4mrD3ETPn1g0J60kTOgc41lEVSqK0wcMLYlAYMgwe+RiHjlyIPx008zICmxEPhFHU7FhULTTp3SsHkSnkNUyPZvh81oH1xVizB+L0PDWHMMAKemAq6XOLNMmgU5I2KtWNjyvSYLOxyblXZxOlbMuWrerUIvrBA0stRU0DaJI5zZAv1oTDzwaPVY5i2BdqGYRFFsp9tMPhXFTTDFPsYmTDtXmNtyED5IJ0/t5DADtoVhtig56i8bkcGtZIrZkBp2GfsK54eYXqQfVF7LpZF4Gjvc6li51Drbp0ULFs1pqqKAiwQygiGHAZIZyPKMNet5ZHDdROno83y4Qh5DRjhDWKfdPKoX96zzWt6HUAZXbccUcb2Tqi0JTNIIQxlWz3XjLyA2CGDqKF4pysOUAPelIuPpYSUBU5n4wSwUqSH/T2+CK0lQdCH6iG+DYa2qSEyVE931vtAHdQcHBBMy92t5x9AxId6m5sLLV0wX2t1qT4wKaK6vn8HpswCrv7FDQPPWMdWy1dMLNc9E/DpllUQhgOY+Qts/h4bTa99KBD0ZwSmvjWGtTkuk78G29AOAuiypsARsVGc1BJDAgglk809IZuNj2bAiPjh5v8qEMgDcCLG9WGjElku4iGlAAABCRJREFUHLkAuAOCfPEMYo/00CDtmgsqW6E7heFRvbzF5s+rrEGP7Z577hk4z82gPwUN1u9TG0rDnV1vC8EC38hzWicOBJES3lLtckQIGRc6wGPCGHIUviBjHIEZ1p/35plyT55z+8wmx1JI0SDZZJ1LHTqzWF/RalvNNjEEZxD5zUSJpD7kwp6COKkldhdFAAjsAqOAB6fCwXrwGsqjXBdeE2A1aoJTHpXWVRgMx30IeAq4DYeUZxpZXdS1Fa1pjlVZxoQoTPsj7EsYdZLMRaww39XGROJ0DHCMOOlCketvH/quDi5vitQpC7t1ZKs2VqzR0sdIvsfDQrGdiyT/heaIM1CPJ8RtwBRCX+b3dNMSZ2pWANRyDm5SHov3jaJx5DtsClfLiKJrPkSMDaiQubAgYbeIytH4oOFJ2w2X8gHEAC/T4X2cYeJe3bVs1RQQCtqE+NLUCg8yymCqplz0MDpuEq6L0hSHlUNMjiTygggGSK24hCgbS/U2Sb26zjSGI67X0mXL9H1J0kr42r0NuIAMAZpcMnquWQyAETm/fJ+p6q5i6WU0hY9hDWJrIjZE94JiBV40IK4uyObPis/HoLjXHNc6iElWWNDrBdIlgkZX8BARVCRS4Nrd27nqSYyEmNTI+4JLKH+UtIxPvZDHWzTsQGMwyBHg4/f5OWGyWFuBcBCVDsWTDmJ/3D+godD08F4YONoo8fQu8ufKGbyXUsCQa1ZDjdm7pHwNJRUj3r3rb0e+tOeSTq4gxdH0yNCdBHYgrAE1yaCGKU4yfduhm4jzQmUF58L94d2JcjylcoFAOZogX4tmG/tAEj9MhdBEDAeAo5H2PdzlQnaP/eKOFofHSxcuw8ILyJvk7eBapn1GEMVyFCAJpTX/pVbWJlfTr3RnAy+YDRAI77CMsHxCfFM+uJeNF9viVOLo7fG2qqSDEIAFHAoWVaADjQ1dPdoIKpHUnZIWPRNWnwdFQo/VxJjMzdH0H8XcHBRjcxNe6nfDOA8PXbzkozpynkZ6R1Mlxr7dRAMvo3iow/vBPeazI9UzDiMTN3e7vC0CRmIJBfqjxAoS8KN9GBjvx4Fg8xEGUq/F8OEJvdifkPdQTTWQBoRkS8PJSxO8P/VRwMRRGq41+DuntVdOzGiZMJOHDeKAYU20RaIdZzT55uKwSQo1oL9+nWnV2+O+KFeK8q5qpaTPFK1r5u+EEFe17c5uB4OIiOgiChK6sfwTh8Lx3jxD1/XyWbWUsYg08Oisgat3NCSBxHvHvJjXy6BovCtRlbf04RBE+glD0/g7835cAgc8Jsw9qjnlF1AxVkD4GSArnpUDRB0XY6TSHNTgJFxjIifmCnmDCsqP8fBHYJFnuXLFCj+ImYwOL85DVMjQiKN6MEO0Z+eUQjr0FWq3lZKrcbAuoRWQn/1fbh9VCp+xIjgAAAAASUVORK5CYII=">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -721,7 +766,13 @@
     <xdr:ext cx="304800" cy="304800"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="AutoShape 14" descr="data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAHsAAACkCAYAAAC3r1GFAAAgAElEQVR4Xmy9B5Sl2VUe+t0c6t7KVZ3TdPfM9ISePIqDRhqhZAn8DMu8hXnPmGXAawHCZDDmwUMYk0GABcY2wQSBSBaSQBKDNJpRGk3OQTOdu7q6ctXN8X/r+/bet+7o+fbqVene/z//Ofvs8O1v75P6ylfuTwaDATKZHDKZDIbDIdLpNHK5HJIkQSqVQqFQ0Fe++Du+n7/j116vh1KppM91u11kUmn0ul1ks1lUqlV0Ox19bjAcYjgcAAkwTPi9XYfXKxaLun7cm+/n/XuDvq7fbbfR6/X1Pl4jneZYEiCd1ec5Xv7ni9eIMfIavC7vw1fcg99zrNlMBvVaDYP+ABOVCjqdDiYnJ7G+vo7+cICpqSmUy2Vdj/95bSRpNJoN/Y3XHQx6+prLZFGv11CpVHQvpNN6P+eB9+X99Cz+lXPG8fErr93v9/X+mAP+rt1u6/7xe36en4n38JHHfx4MbL1qtZq+JgO7ZjabQbFYQurRRz+TJACyvtgcDC/A/5zAmKj4ykXW4g046fZ3CklMLNcAyVDvyWSymkDekO/JZCgIPc46uFx68H6fP6JSqaLZbCCTztjkcuFgg09RQAYDDJNE10mlbHIyubx+jjHwPrwff8eJiYnm2PL5/GjSY3K5yFxwjovCx89SkPj+drercU9MTIwm2+YgrbEUikXdo9Np6bq9Dt8/0PizuSz6w+FIiDlPMU6TBKDVauna/Bs/z+cZF8zYWHr+VErvp4A1Gg1sbW3pd5VK2TadhDBBqWRj5TU5tkzKNif/a30eeeSzCW9EqaBUhzRmMiaNsWt5gZAwDoSf4QXGX3wgTjDfpwE2GppkLn08kIQ+AbLSHKYN4sFarbYmm/fkq8MBZzJoN1vo8/tsVg+RzmYwMzOja8YYOAl8qPHdHRPJa8Ru5vslKJkMEkp9xrQDBW44sPFo0pEaCXOz0USn28G+ffuktXRPLnCvp89QSMoTpp14T16f8xC7lb/jz3x/aAj+HEKgsQ+GWshWp439+/ePtGyMnfcZ9Hsab284sE3A3ZskyOZMI+dzuxsxFlnP0uuaUHGxbQdkkMvGg6eQplhwx2ezI9XDwYeKp3qhpPPv8Qq1rxtQLfUHSHH3+04P6YWEwXYIP8Ndwr/x//b2ttTOxEQF2byZEk5Es9mUFOt+aVPNMRG8X71eH/0cE8txUfXHK8yGFjpJkKdK5GK128hkM0hzTLwfhaBQ1L34GalvQIuhuTIjos/SJHXaHZTKBY2fgspdSIEYN4tUrRT8MIn8Wwidmb8U2u0OUukU8oXCyByFidI4+n3kc3kMYLs1TClNCe/ZbpugmrkbjjZNMZ8zIX7mmYcT7hqqU74K+bzZwIxJTbw4UP6ev6OEUgVJsoecexOOUCGyYbk8qKz5no3NdQ2CExFmQjug29X1ymWqnwES3xm0vnpwV/cxCqp1jqPX7vBxkc3nJQSctGq1OhrruI2L3c3J54Rwgig81CBSdy5wOZoPJBgkplI5YVxYCdtwiKYvYJg3PsfOzo7uqUV0/6DdbWsecrmChIjCzvmlLdd8pmyhzBylpJK5cfjM3ADtTlv+QzzDxsbGSHiq5Qn9jf7EuGngfIdW4XxwLkJ1x9+kbb/ylQeSMp0E38X8pe1YU9vhjPHBeSHZJ19sk54JORJUg8WiSbfZNu6+oSai26V6tuuFitNuGZrTw50sByudNtua0KY1sb21je2dHZSKRRw6dAirG+taBNpH2ihKeKjDuG44llxYTmjsjBi33i/NQ7tb0PWnJie1O+kzFMsVrK+tI1/IY35+fuRvxFyMa69mo4Ecn6/T0Rj17IlNfKfTs53X72sjcY6pwQqFnNQ+BWVlZUXjp/ks5vJaAy4kf8c55e/54nzKbGbMNNCMhXaKv8VGDBPKcfLznA9qPdnsxx57KOGH292+VEkpbxKdSnEf8UY2aDpwox3mNjkmOLzyojsLcsiovodDPSQH1u31sLW5qZv2B2aLudgUECrJGKQW39XpoD+UWjOv1zx/Si2FiLuF+jSdzqDb77k3PpQnigGwuGcR9Tq95kk5W/Ja+wOZjjTv7d5uJksHic5kHu1WC8ikJQx93y0lqdTE7pGixkvrs7LJYcYonM0mVldXUCwUtfuSlO14037uZfNGqZTsLn0AzpG0B4Bex7QOhY8CxMXms/Kz1CKT1arMDl+r6+t6Xr4nbDMFM3yEiFBC8MOZTj355BcTqhpkslJFGdDB4ETa0vZ6HQ2aaom2iu/lhHJgfJBQY1IX3M30SD2Ei5Aq7DE93xAgqTEP7ai+5Xi5d08JplXs9xP5EXxY7cApk9R+zx2gQR/JMNEC8R5JYiGWpCexHVEsFTHw8IxmI5fNabHtfnwiap8ChoNEO3B9Y10LMj83p5+7rbZMVofOkdtwOUU+rjATw56ZQfkrFNi8LUy300V/0Nd9ad/Hwz9+Nmx4q1GX2s8Vzcni83CMVPGcf96v1WhKC4bDG+8L7ztsdcyjaVWLKjS2Z198IqFNkgT1uihkcpK8YWKhQKgLTjofIn7mLih76KAwhwvsNl5T6HFpSLWkjB6jS608U9nOtNSSpLvXe02IRBulsML/ZuaFXrTZPE6IHoKeJr33rsX0nFhei3aWO4LPxWeKUIy7k2q81W5pJ4a3TO3DBdGOTZuqDDVqiwp0JVR2fwvV0nouhYa01VzU4RCFcmm0q/nMNCvhryhUpUD7HAlTGPakbrm4IQAjjZBOj6KWcDLNL8iNsIoILWOueL/Qlvydnv2p5x4RqFIulc1uwzzbcqkgCTdny8IVOSeuiqhCQqJ4oXBcQm3JexwMMOngQ3jo3FUCWuiM0V9JpxRiUUVxYSOc4PWnJyfNi4Q5TXpQJCjkC/LaeX8+JD1pxrdcKKp4TmIsFEO8drulxZVJoK2mk0YB6nYNtODOd+eQO1iefio9MkXUAAp5ej20uh19nhM5HkoVsjkJlRwlmqGUCW84TvGZiGBoMrtde26Fn7Is5vxyTOHAUaD47KGyuXBzc3OvCWUjnAuVH+qb742/6XpPP/eogkw5LcMBCrk8mrU6si6hqbQF5IWCxb5STZykUsnCKk4Mna9koAGN7ARBAvfeIzzjoLk4dPT4PqpIDmK7XhvFvfzM7MwMWu32KKzLc6L7nDhDybiLqRppTkpFQ6K0A4e07ebwaVe4g8j7Npst/Z0mioJRqVb0lYLNC3KHc2KlGt1eT9BLdmSO9+ecMIwUltDrax6klRJaDQN6KMC8Hk0HJYoCxleYNOogaaFOR5+nNy6zZ2/D/PzsSKOG4JvDa6/xWJ6fD78gMA5uAqGh6YzubethplWLzZ2hsCABOq02qpWKSSehR/q83ClpAwG4GNyx3DGx66QmcqZqAjyhMNTq9dd486PY1uFBugU0B4VSUXZ0HC0at4+h8kIoQ7VucXfT4XEAQ0JZNGiXoZs8dtdMXCyzm4kBNPTUM1TBpgWIehEmrUwY3KmFpOYo5PUzr5dn3I+UaRIHXei48aXQldfu9qShKFjTMzOjiGZkN31M1BS8PwEbLUqhgEa9gYmKhad8hWoObcnn5FgVkfR6Ei5uHL4/5t6wCEMWBU7Rdxmak5h66tnHkoBAOVmUODpOmXQKDC3MVqX1gFT18pZztDe2k/h3gg0UgMCF+X6qND68QhXChfLOzRSYM2UOoL6nL0CwJLHYnrY2Yn/6CozZOdGESTWRdK40Jj68LZjtPBfIlMW2HCvtOHetoNax8E82t0sVaVJvCF0GRPEYslBI+FwMnbhr+ZwUBMW57plzgTkHfF5BpA558rliXqYqVY2NWobCymcNDcdn1Wd890tTMqZniOvQzfT0tASJG5DzEoJuzrAJGsdvttxQtRBwrolpV4tkUi+8/IwjaLsgCgdEEF0OBBfL1Qe9VvNg9QtHwMzrJfTJRaEKlQfoi0nEZ2NzwxElG8y41MbgLTGRlwoM3Jzf2QLaAyREy2lfAallhm2cVH7WJm4gf0A+RD6vhSKerJ3q3jd3KLUBF1DXSlnSRzsjbQ6p7bAKehJYe1ZeK9RqxNpyHtMGJnEX8sXvhTJms2hw0YQZ0GegYAwVj4dQclEnpyYtOeTTyvFwiiLMpRAqWnL7G5uEfku9sTNyOu3vKdn78MCZhyBIQ8xEavyZF59OtIiZFPIZokwNvbndaqBcKGEw6KPoWLW8c0mK2Sg+kOBFd3CUpZmYGDkFFBpqCmZcwqYp5u6YrZH5cODGMjp5CY2841xOmoVj4TWofQK14wSGdqA24WfDWYoIIkIcU30ptDud0b1kagbEx7N6BoEghCzTad2Ln+H9+BniCwZYDLBTq7lQM2IxRDGik1TWsk0Ubl6bfoZ2snvcMZ4AP8zh7KM6NWXJIvoXBT4/zUxfmkJ+1MCwBjqTvP7U9PTImTREzoQtwmD+bmS6uhQUcxilgV4++5KEiCBARmrUEBxmcxT0p2jPbUcRXOC2swU39IuCwt9x0gjtlcplhWHh2PDGdQL8zaYGPlGZ0OcD2aIzxJ/lpPCaA3P0qpOTI7+B15eEc9CDvsKi8GojpjR1Y1omJpYIFe0bNUCn05ZfEF5xqG6ZBU9cUBtQi0i1e+aI9k8qME3YNJGGKJWKSIa2kLy/wKVCVosRjlK/w4wefYMsCDYF3Mz3M2oggra1tY2Oe/Czs7MygxGXB6bPZxF27iqeP0sQ220JFneurunp1LDdYSIVy1PLyWY//1TCC+RyWYM23bGhyrTQimogh/Qw0c7iwwp6c4mykMrsnh6eNtRVeG1nR6B+2DA+CCVND5LQqelJYmWvlRk1eJYf53hGgMWQKnoXiTJNZHlzLmAAGgrhaNv1ecPCeT8JL737HLFuy3QxxuZX/p2LaGAPowWOlwtroVOnZ37G0L3xiCzCpvO5OW+0n51O10wLkbY0Q7WugKq+A1S6n4dk/IZhF6OOgKQjvOQut8RMSiqcY+dzxqbgnEYoK83nDhqvR/vOr1wzCgId5Ugppx596pEk0Cthub2+FpXOkGDPrCUMUkyMM1HiMabCINlXUyN0lCSBvnDcoRQMOkemWgwjpvetzJDwdMavGUkdFzqIArHLLRwkNErEzAAOLgr/zpBJpoC73L3rVqcjIeHc8p7joQntI69BoRHSlBhAxPHH/ahOI1mTTpl2IronGzow7TaO7UcsbOrUEibUVFqklAMy/S7o4kWem8/ATcB5irCJX/lZjpfzwu8j8rFM3FDzzh0aYaG0WJ+hZl/+CZ+DIhs+Q2g5aVHOMX2OrzzxsBabEs3kAzOblvUpyIYw7JG7z90c6kJwqKl0hWeesjTPkHivQYMCMnyyeE3loxXSEK60XTk+6GBtmP9HreK5Y4kZUKvtaLG1kxxk4b1MJXeVaJAQuoaIxRMY4lkrM0kWr3Lx5StwEvs9MK6mA0cVST/DQk8TLu2uMUcp1HVMrrJ2SSJvXlEKIxJh8gyxnGDhmTV+Vo6TmxXZW0LGLoiBuMnhYx6AGEOwcTx219iYMWQmMaITwsaDwUhg+RwCv3zTpB5+/MsiL5hX20POSQv5vDkuXGzFa2RtkHLjoRQnmw+hz7ojQlvHvSc141SkwMM5cE4Y6UWUQEocU5sUsJBCxdF8KAdPtOMUqlhYRc1gnrQtgMXLWak8MyW0nwNPF+6SLwK8oE2kAIQTQ01C28nPa/cS5iyUNEFcAD53eODhcYd9DHAj7DavG3FxhEImtDaO8C3CxDUaNWmY0A5M1hAj4M90TCm4XGgKJ0OucAYDIg0oVQAPYWeaNUfslDhyUItaMfyY1GNPP+pMFYt9mSDnhxrNuhaYzgWlqpwv6uE5iAjutbPH+Gjc7bSLyiyNATDSAo6XCzcfZc2C/ODok1N0LMzi5Nv1OB6OY2enprw3BaxQKJoal49AEoGBJYwciGLxPZxkqr+AGyNRMA7YRMxLdWjYQErXpSaIxYisGxcu8PtwgGKxKbTB6qGm0AJ4WBhUKQoRx8+IhQIsP4SIH59xLEbnNRk2hRMs6Nk1JXludHjDBNIp5Pt4T3EISH4grE2giBh8Pi9TKij3iWceSyg5TGVyMFnu7I57fz2qtJYgSdocTly+UEK5zLQl1bqF/nzI0A6GsBm5kDtcUF/CHWuYeAAInHCCFoa42a6MGNESFvQwzQwo/CAE6ULEh+N/20H8m/JAcro0CQRcGC83GqOxxU4Nr5XPKgH0JBCvx8WlL6A42Yl9kXjg89GX4c+2aJaIiMWmg8YF4hgopAzBNzc3R7loOYtyuIxXJ6zdSYYUNGooJm20OMp7M09uiKRsuzuIyk0QtMmksbOzbSEI4+uJsogYEcJFXB+OM7GD1Jce/aJsNrHtGj88HEjd5tMJup22EvrJYIB8sYRSqYzSxASq1UmUJ6Y8xKKDYyqf6pA340LRVlG1cuI6XebELbnP0IYTJKTO0Z7AfkfeKBGxXneESAkJC9za0TeaAJoMjr3bY5zqSBi/IoASU9nKjrmpUa7aKVAUXu7+yJ5xYiIk5ELyvzYA05m9rjhoy8vLyGWY5m3ImYpEBdOvBw7st3yBzBnnxeJ2vm9udlZ+TrNFUqUJI22tOZ4MpxjimQOby+cUVnEHVzwCoqqTQJaK0mB8z6WLF0zbFkpm5sjedSda8+Kw68hmf/mxLyX8ZaO+g067jmGvIyZIPmcTORx0iOojRQaGXPoicoUiKlML8gRJdqA0kiJEOHUwNFQqGCfaCV1yy7bk/Fy4cAGLiwvYs2ePecEOH9KeinjgryAdctdzh8euNrtkSX9OEAkKVOMUDl6P/zlew9oTQY8kSWSFtqVQKhSxtramu3CMAUhEJDCeOQo1zK9rq1c02advuwOf/Ohf49a73iCHs9M2XDoyf+F/MKdgmT9T54pcHCfgV+IOnLdxti43bbtlISIXmxrXHEFuImozmxyxiJIEa2uGIzBvwfmi3S+VLWFFTaJMpUgWBqumHvzS5xLyoNu1bQx6bXQb22g2ami36yCLI5fLmFpk4l057RQq1UkgW/IwKytUh7TeoiQsh3K5guGgj1azhYcffhhveet9MgecUE4+NYFiWIVK3EGkPNmDmUNkHjOFicTDRsPIhJxsqubAyvk3OljdbkdmCJ6WLOSpRSioxptmOElSgBZ0OJR65cQyAgmTwPtywng92UDPpIWD1WvXsLm5gTe+5W34o9/7EN7zDd+MhESO7Z0RHsAJDQHu9Q13N66bRR1yNDNmvgwhsx1Oc2eQr+EMNJvUKPSsFW45Pp9JG75BU8DfUROb+bHsXIZhpwSKiaqszKbRr90UfvTjf5Vk0n3UNtfQbzfQbTN+LYgmw1evb+nMtHO4h4yrBZ4QB88jTbJDvojiRAXF4gRKpYoGJL5VviDItdHpeVrTmBOBo9PmcMEIhHCSRdFxZC5if+4+Tg7NQLvbcWpSRfE3QyXa2Ga9qc9ZmJdCtcpkRV8U2vg9J4PcdArG1tamcHZOEjNh/EwQB8JciF3rW4mfbTS2UdvewA03344/+59/gG/51n+jzygJJC/egB7aawpKs1l/zZgsvcp8g6U9RcaUo2lzIoFwX4S7lbtaCaLQViOMwVk5bhKEySeGFWTyTEUXTJspbBsI8qVzq4TLX/zZf0u2tlfRqW9idqqCen1Hu6TXG2gnKF/NZEQkDpwJkmT5YMwDTyBfKiNXKCObLSCdLSKTy6BanRKVaXpyGps7dUPcFN7Q4zfHy0APc3I4mIhZd4n+fVQqEyIMcFE2tjZx9uxZLC0tKQ/Mscnm0oZlcyjm8zh27BiOHz+O6ekZdFpG/Y3EA2Nnzjb9kJ3ajpH0U4aARXjEcZjGsR3HCadz1GzsYGdzDdfdeCv++i/+DN/2r79LGiLoxeMevj1P1xiwYv0MtYvDJ1EWjQkPX/TAsoMsEk5faDja+OAO0P5qw4CgEfPvpEQXjXiS92oRYhTOy6P/QPuukPnDf/rBBANOWBubqysoTzhJYWjlJ5Q8euIcSHjc4chIEDI5qZpMtoBMlra7gHxxQna9Wp3GxOQCElJkCcP6i+GdqjGodpBCd2ATzAdReU82JwDlxZdewksvvYS1jTX9vecxcuzWcOzGVfHoHtz5JUYPBczPzOL06dO44/Y7BOoEZYcLFHbbgKTirsOWSrQjDB2DdnV9Yw2HT1yPhz57P97xvm82E0LOuUyMOUfhW9Cho8Mlm8xQivj5iPtmi8fn5e/DmVVenqZnQAEzDrrSlA6bCqyhqePadNoCkoQRgMCNcpNmNpywqSSVo2rSJb/xKz+eFLLMTfeRY/oysbonVmGYnbGgPC5CO0Q3n1IXjpI8cd0ASOdyUunZXBmV6iwW9h7FEAa+iKtFe0ywwGNvARwYKmy5cPkSnnnmGZw5c0YL0uoZm4NaRQ/ioVKABLHYoeqCIBDhEgkVfHCKFBedCRSmGMnEvOmmm6QFIg7ns0Y+X0BFwsXxWjKyaTZWsbp0Ea+756347D9+Cm++712iRtEfMNNjfLjIm9PTjjy9tJrnlhU1EATSHBAM4WLtEhW5Uw1MIQ/Acp00WSJe+m4NoCSfI9RMoqcnnpwzyKRPVI44XGj3+LX//P0JbVKxVECKnGXmdJkA8cUhmCV97xmeqMXiLjCuuZH7hCwxFOoPMTk5jUw6j/LUDKbnDmFyZlG5XQoMUbrI1jIuZCjz4osv4oXnn8dOoy5HLZIe8mYdirUFNI6a0Qu5YUzqRy/BmYwc7DchFBa3GzrHF8fBsIg7l/7I1NQ0bjx1CqdvuUVJlYjh47r83M72GlYvncPb3/3PcP+n78edb7pXBX6tesMWeWglReZMmXOpHcl/TvlSalh+gKlxIYb8zMDoTBEi8omocZjgiKcbkFYfxZBD80+4QfVMJC24phDsyhwFMQg3vYFmpn7xA9+TCIhPBihmWQJEN9/LdrSjzdBzNxIrV/VleIeUfDkkeaRdBXECaZyZCJia24NuUsSpW+6SNy4MmA816GNlZRVffvQrePXVV9Go1XVN2mYLxQzgtwW1laMW4WLzRS1iEmsPPVLd/n6S+cY/GzYw3isChvLmNE/GvEwPWVxYwVS1iltuuQWnTp0aZfc4ofXaOlYvnsPdb/46vPLyqzh2/U2y2TQtlrbkeI3kwBeflTl5YeacI3rVjoFHrK9lF2c9IyxD8XmAJq6OhRYWC2hRZauuwoTF5sTSzj4tUtkULoOxeyq62N3ZKaR+6QPflyhWywJDJh6YRRrS1hhFKQj7uyGRTbAyQp7jNpaG2fRR2pDFe4UK0vkqbr37rQIWRLYf9PHZBx/AU089iWa9MWJNWrxrFZ0Kl9xWxWLbw9kuEanPvW89rDMzYzEJqkilxxZ3Idjd2TZ2qVenKvNnyzkbIsg5IaBx04034fbbb8fO6hWsLl3AqZtvQa5YRaFcVdIj8TqrkTlIGS1bfgSdUa6E72gOWz7JWHgU8KuhjtSNxgW0/IFlBM2AkZJlSBsdM1HFXJOEuFui1lBN2/l0DFmk6MLxyz/3/oQDK5XzSDn91x6YWbCWFps7ke+PhAM/Ssg0dlxUUHCHh0dN9d5Psjh7cQXf9h3fJ/L9o08/g8cefwxXl68YgDJWSx1o2jh8GQscO9cEjjvbfIRQ7UNpZ+On0QSxIsScGtMMAlrGXiEUIUghWJaZM3iSU6a8fS6DifIEKqUK9i/M4NSNN+PW2+8UM1aOnlivu4wUwqaMDOhAEZMWS5Z2WaQI2wzyNZzRqw3j5BAurmWwGN6akFD70L5TG3EjjFBGpmhJn/Y5ZMREDSyOn7Sikys4D4Fs/uSP/9ukpKJwMk4oUgPk6FJ5WQztIyU0EhvipzG0cIaJr7iQLKnYtNVqK8eayeHVy1t45zf+n/jkpz+F8+cuaCe3O1TpVpyuHUYO1oi44EkT7TjPJXsFRnjd8uG1K6nGBhh4sZyx12yhtcjK8VqJsNlHI7jF38eFaFybjAtHwKb58gQI1jA+J4tmfmYex6+5BtccPmDeL3qkfouuJIFNzLHV7vTiwVjgKPYzgQzv2ahFgmY7lsAJuJNzTY89dr9COdaBZ4NGxXsa8ZGOXEC8xrBJI0XYlvyBX//Vn0zajQYmq+Sb9QxtoipKvG56wNJQBu4GBngkotooedJEZ+QtkqFhD6b0Jx2GXBk7/RKefv5ZrG1uIDUw4iCxbNpk2maFcz7rsYBhm2PhQtWG6chI4o0LpyyYCmK4iJT0XY41d7+WX3YuhVTGhGfcnsf3sdvHfYBIJ3Lxc1TtBZL3c0bu4KISfi2X5eFP5LK47fQNmJmwShBqiBFU6hUZdLgshbtrPhgDBz4fwEqMyWrJrALGVLz5TwRvbOGNI9DvGRaiOfDUcrBc+DMxc23WD/3mB5LN7XVMVSYsC6UkeQqH9h/Bvn17MDU1o52aLVWMJeElran00PK+nabiPe5WOhgE8pP+EINCFc+/chYvv/yyUpO0J60mHTDzsBV6yNu23Rn2OB6Uv1eO2RhyI0+aP4loPyq8J2Y8MJanY+KBfAnpc7LguJMW34f61jXdU9+140b0I0TJF/EDZIj/M+WbR67AxFBJDpbsvfyeDMrFKrKpIfbNVnDztddKEzDC6QtYoa9jzQqIVyszSIoVee6OM3Ac0nhjPooVRXhRorho1q4EKdvhUTYdqePYHBIW2vVg5Xz6H/4k6XaZ5aIt6WN1dVWkAuKvlCLaHbryzIpJUl18xIPOpOTFmlonamRgQJLL4eJmGy+9+KKcLg6e3mGzaYjPSK0ZlVrvsV1kYU+kN7ngI+ryWDWE/C7PiZvN4mJzZB5aOcGBJsfE3VKioSliYcMsjNvzEDZG/0aiMEdIi6SEQxHFUkVZQC4UVaS0U8YBGAqiV8jksmkUc1nMVSq45aaTgobTXpJLZyvoybLPo1IdY+2qqsRLltR1watCtEPdQeYGi9DLtoQ5hTJhgp4jXrcwL/UXf/RLSqdQCsx+GrbLeqSwlLcAACAASURBVGVKEFWFpQB366t5MzpYVD9cSEuRplApl5CvLqJXrOCVl7+K7Z1tT/dZxobCwCR/qGsuWDgY8RASHKFK9PAt8xYPZ7nrFLIeUlAABfprt7CyMoMBQ5mITp1HF5LOz47b43FPPDJc4dD1B8zpm2PFCSSOzs8TFqbJylcqUum5gvVqSWjC+kaUVIHgwHqqsFxI8zrsygGeLGXx7ne8HSxl5D1VvizqtFWrBpUrtJIxTswkBMxqxY6SeOcAmh/i0qy/8dmiPs1dFqR+4xd+ILHuOlbiQlBBXQdy5FSToGDeLKmzQqpUOG/0YpHbvc0EXaFBfhKl/dfiqYc/j3q7hW6LjpgJCz9HDjZBei6MFtE5zrHrAgkL7jYHH4BNCIF2WYQXopsx+LTnlKOUIZ7kxQgeesX1YyG/NpwLTRM73cIWCwNDy1CdcxMYPFxEkiNzp4wkYzufQsD38FqCdj3lmvI0roiVFM52C1tXL+H2G6/DO9/5Ts/W2diJZ/Mlb97JFRKUsZKrCKtIkmDVjsHYHoV4XxjLqRv3PIAcRQS/9cs/rG1n5D9ic27nvPoiiuRMzbgO99KfiANbrR0MhxnsP/12/N3f/SUyDnZQOxiNyJiTzDoZB4w/m80Sb83VdYRtob7DBsm++w4Zt62pUH9qCUVfg8O3/HHs4PAFIqQLJ2/cRxjH2GMMDKG0WxyNE1qo3LLVUTHTx8RPJl9Chg4se9Kwhj2VQb1hiR9OGGu4FF4hjXTSQ7NeR7u2iU5tE//ym78JJ48ftbptItxO+DAGi5mRICMGrs4oRxx4gkwwGFUl6iRDiMpkcxuVNJFdUzLlv37wP2ixVZfsZD05JE67FewmgMOACM5vgP02EH4uwczR2/DYc1/F6tIr9neVsUTLJ7NrDCcaDcKmJDdSEMx+M24OdR12VWqIVZNy4v7/VYzane5lWu2MIUtc7FDX4Wz972x0/C7s9bizpmuz84SXB+k6LlhRCWI8vDzSuRISpRfJiSvK8TThNAezXGE+voE+bWmvo2Cwtn4VrfqWHLef+g8/aowez9eP8geROxBl2KBYsW2UhevLUMlNUbxOyNXyF7wW7z1OqwoMI/WhX/mhJBZUgIX3BIv6qmBXWALe0pPuH5tXyf+dFvLH34L7P/a3SIYNDZxMC8F3TMnxMwJDDPK02m4Lk0wN79rmcFSsPHfXWePYYkxRQWnjME63TJbHcKGmww+I3bp7bbNv8dz83jJ4RpDQriSvzZEv+QxU105CMNvpoU62YOYuV0A6V0QhVxSIwQVniljz0++jTnIGG24NE2ytLmN7ZxXpwRA/+1M/6R0d6MgydUmVbpskiBARchl2bhiZxeduucliCQfWKckjs0aNOCTjN4/Ub/3iv08YQrCaIfhhu2GPYa8RAoUDZ5JvO55aodnroDZ5E557+CHUayvyUoOcR+FhJ0LtdudHEVMW0N8xcgFDMKk6955t4i15Eeo7FkEL57zvWLyAH9NZW0Q5bWMtu8a97XD2wqEZQZtj8Kny7EwFEqgcYdVWshTqn0V0NqHuw5C/njMiZrqQQy5rxREZr4ztscojGQgf315dRr2xjnwqg//4Yz/ila1dLSQXJgoNZJfFErW+K9FKLNp1EBs3pMyRNufnGZpsXj2/mgYGUh/8T9+nKk5WPoSBskm3zJDZM8szx1dzZAylYrhEqtLmxLV49itfRLOxpsExqWDCYzsyYL4g9wVRn5+ntgjnKHZbnoUEASOSOapWGUZb4kv23MEVLTpBBu4cx8/HwZH4Pr4K2Bgj/MeCh6NmKt18F4Ieso8Ou45/TuPwWD6XLig0Yx6/n5D4UGLnS5RLJEZah0JmyQrZNDZXCRevo5jJ4Sd++AcdLbPuipayNAdTIIwDMOGoKUHkfsS4mQptFlrMwBbWirtW5dxxsWUPnPX5tZ5qEP/dr3fyn4Hz2o3suNDpY/KGd+Lxzz+AixdeRNY9VO5wMk0M6SJD1CoUgjhnHja9cgM1DB40ocupoJBCZa42Q6qAT0cPOQb6K+4nNjDWqoPPFQscKjoctPHnDOctBM5UqAmVFbfbDhnVTHmZrqIRvx93eIoOWybHDJChXKRZFyc1hiafvdVGIZfG9toyavUNlHJ5/NSP/ahrNIIO1Epm7zkHyi94nbnh6bYfd5MlZsi4uagNhNx5HkB22pHMqC9P/ebPvz/hgKluwhGKna3p9fAodpOBdmzlZIxKJgJanT5Ofv2343P/9ABeefZRZNJUw6wVtvJdAhGhsg0T52TKuzDKMLsVhN11hEwqyEOvcDYi2c8HkkMXjXr4wKL5WLw5WgDPzH2tGh/f9eO7elfr2K6WgIAolJVARdGinM+BJzBYo6XSHysglLOWNgHJ5stC3bhjudDKQPXbqG2to1nbUi79R37g+1+jrYLepDVx51g5ctcsMUYrLdrtLxsmRqGqGEAUxF1QSprhN37ue9VAx+LBcFJMYsxT3m2foR3mHYXDzhK9ajVauO6d34Gnn3gWzz/xJXQ77NhgHuHkpBXDGxZuVRoR+1kmJ6V8dixQ5K3lhHmMKiKe57HNSfOiAW8UQGecjk/kt83W72a75FX/bwraQ+XLprmDE9/H5JFLxvdxh4emkJD3jDOnZxqShWPv0SKl89o8SOeQVTtN443xvflsVqyXTquOublZfO93faelI51PF4Idv4tx8e/jYwuTE8JhPpDVltNB5L2ClxDzl/qVD/w7lexavbEjVGNNVqN6kQ8RN+CFFhYWwBYQxWIeSSaHzuQJnLu8ise/8KAexpy6IeYXZ71wwOyWhVKmqqimVNM84lPvdn+IQgOOje0raYMCD4/sFheedj0ctkhphoqORY5F3Q0jvZPDGGWY4+JzRQgY6jBaXkdnhQA4ct5zRmgZm+8RIVSM7w1o046sSWPSnzVGSqrLxj/b4udff/11+OEf/EFfbGO2hJNq/lHAqJ5p9HZlaTmHDDONYxa1cdS6mltH56h9ogpUc/BLP/OdymczbolYkzsnVGXknMnbYq8RPvSo1ssTCCwZquX24NIO8MTnP4Mrly+OgILyBInwjEENFQpEzXZL3hrTpq2nWBD+xu1sOGJmUkIhW2Jf2ACT/DExY4iZdp+XvgYuEJM5vtPDHkc0EL5DaAIrKjRGy8jR89BHvVy8dZeySwlZKabOuU4K1cQxy6g0R/dXjqAuuPRd73o3/vk3vHdMjTMnb+2/FPJGaOpOqXnf5mkr7aww2Xh9Rllwe27fjHiC8WypX/zpf5swSJeKYTG351S5uATuc85bjpCF8bEe2u1jmlNNzzFVwvnuNB556LO48NWXkMomyInUDiwszo2AFAvx0t5vu6ydHdpDu9ix8NiNoY7DpBAXd1/JAIxUImGx1N5uY55Q5fE1JinEJa7Pn2PXCuN3vH40qeS5ec45FtxqoS29Glg2+WEquqcL7tGCqWAjTrCXaTTwEVU6ncKHPvQhlUiHmRPbhw7pWBp2V0CtBp73NQ3rFC0nMHCiJdzeL2a0+B45aSwf+In/OyFXiv27SbpXB6IRMS9tOLSyLN7wLpIQUYutBu9ZdIcJznXm8ORXHsa5l55Ft99GOrHWUlNTE1LZFDcurrzMPqE9a0jL3msGtJiHHwAHB8hdoqY3rE5UV0Dz3G3X7qpxg3stsRI7OhY6zAavN55wGXfUYnF31WhMqoFIRtm1/IBSvS41I+dJZLY0uh0nGoYdbvdUkkP1ru5L0XigVMQHP/hBoYCGVnr1ihMTuKjGOHGKkYeD+tmTM0ZiMAatSIteVGkIk7FUhcwpu5hC6o9/9/9J1HzVS2eEgdDekBJM58JPGMhmmOVJI3EUiQsshIv9vAg2II2vrnbxwvPP4qlHviSCvvBqVmeW2LzVPPKYVLOPhhoV8+wRYrxyld96OBOLEwLAWnH+jTtZsbtHBru7w9E9j+3Gw6zxRRy/7tdqgLh3CA0xcj4rd4xahgRI4YsgJ4222Om84deElookje1QFjQaF+/EyWvwH37sx91OBxXZulOpfwrDWmbt1FLL1HIIp1KqhRyGHWeiOOql4zjU9M+aBFohgiGRCls/9td/mBTLRWTUSwQCBZKEKTfr2zGi73oFQ3qw60QpNEmxwRtj3DSu1od48atn8ehDD2B1ZWmUiy6W8ihPGJPFvHEvuAtb64sbPkOYknEHSw/oD0xvM4SGYyTGzOvGZHxtDB3OllKKXgfN7yMBIgFyGz+uBew6VuhOSFRC5zy34I0x2aNIIW190MI+mgOaRTIIO2u5ezstIY1f//VfwczU9AhsspbfFs4JKQvbzHvGbg/AhbaakYznrpW/GrP1u2RM3ziujVMPff5+IX9q0KL2y757vGwm3H2Lei0nPY4hy6HxdFo/yeHxVy7jSw/8Iy6++qKpmEwa+VxWhQfRp4XccF5OdUjFDLpt6xca6pkTHs1aaU85iVTz47tw3KabJTPHJUKRWPiv1RKx2/lc4/cct7OKSZ0gEOxPYeXBb1NDH2eQuhYZjzLsnhmFWeY505QbCklG7Xd/93fjDW94nXPw9FcRMGge4h7RrYmXFzVpnA3rfPQe07DUKS64chIpcKo5G8rsGcnRk1kPP/JgQk/R0pykYxqYMALhnWLbb1uXWz6keeNx8k5KD8JS3VyuhOcuruIrX3wQLz39+AgUoNQyfjS8mXnznpAhkeDTAyR9CxnGqzPi4aJOy0AZE7RQw5EsYYO+r0XG4vOhHcIPCDX7tSp+3L6H4IzfS8wVz+Pzmv2ehakhMCEs0cFR3HkdTZHHgYMH8KZ77sGdd95h+RWRRUwTRe6BZkkOn0cQ0UslFt9Ewtil9PLDWbOMJVG0XWbqeMtt81E8qfT5z9+fsBMv7aHVPRmfigNSAl0XIqmcRXQseLOeXqxgZH5a2DbhTZ2pUcCVtW18+nOfw/NPPKLUpXUpsm75LMfhBLJVRKdjvcJZE8XidoUT8jDNQYtJCE95F3TZ7T8mQqEcOscH8plRV4TAv3fBEXOc+IpESahsmYgxtC3MQGiPuHcsfpiC2P1a9HYfe/fuxfu///2iHhsM5Pdy+rAEMG3PZxTh3TGxr7uIEuwU6Y3reV+WRRlgYk2AeS91qnAiYtC2rJWJbRoCQcIlIivorcVSD372kwmzVjqRJ2vdh1l7FQDEoGt4axSuST2pgsT7blLd+SEtjDFT6QKefOUM7v/E36Fe2xoxIwnAWO/SrOq2u11SZ62WizaXLzEyHXCJiYoJjh0+PtFy1EZJGh65YDZzHIXiIkZIFRBo7HK+N8xULGjYXA1ojIgYAjCeJ45dd8cdd+DffNu3e67AKjZpQ6PG21SpF+2JXGmYugmZVW8QhwgnkjtcvD0nDHLhtHO9k4L5GAyTdxeVi22JKzp0Rhahn0EBoGoX+vfpf/ibJM3QqdPWLstn85icncYLzz6FYcIwjJBnFXv37ZHtaNU3MUgySGVYrZlHZgDkK2wIYwxPqphXlrfw9x/9G6wuLwlDZ5E4ww+q6Xqt7g3r2BfNeoMOKInOlFEI70kRIy8ECXG3VktxtZzH6LliNnZ0ksAYOTGw5JjIWAC+N6jIdoSUYf29riF8/G9CbdpGCQ5f/NAEHCfr2n7mJ39KY2ZhgHqjD/qqTbfEhqVbWYynpvYD48rzFa1GuLBEIlUbzoZ9Y3kBnVDk7SrDbBCNMzqxaYg0mUHhs+ikBeMPcvz0j4zFk0Lqr/78D5Lq9Ax63bYkgdX611x7Eg/d/wkcP3EKi/sO4+WXX0Q+m8aBw0fx8tOP4/ipm3DxygomJyZw6dXnkJ+YQc/JJCwiT+XzuLzVwSMPfUYdE4kzVCtV84QdoCB0yvBASJDiCqtdGn+Zat/9XahNBXoKKSJDZHlmkiNjUUMtj9vmXe+eMazVnekeHpoY08N7sPjC8prjsWqo0sgw/b8/87OYqU6pw7HUvldi8Hk4FoavfFajEVGT2PtCg9gzMS9hVCRRmdzzj0NtKDChUaTxmPpVBMDuzz2rvuUpB+xVquY6lofv+r34GYFVH/nw/0hm5mbVe2t6egoXzp3DnXe/Dl/8p0+qo++RU7dgmcXvVy/h+tN34IXnnsDJ625Coz3EwsIcHn3gozhx+s0oqEVFHfv278fTX7of5cM34S8+/GEsXVpCPp9RO6geC/ac6cLJ4aFkQnpiQcc93rGFJl4VvTsNVCHQE0wWS4wYkGKCQVNjDppXcnqXYOamJQyBKbN6xc/90G7lzus6Bz1Sq9EiOrEMHR1F64OSYHJqGj/3sz+npEh446ERgnI1KgOWX8IerB3tYIJNpkms0Q0PYlPNupMuIoyjsLIxACneuXzBKkM8VCQMbfQuo25Rm/R40kGpKN+l06xbXThbpdCGs/PC3MI8dra3MT+/gLOvfhU3n74Vzz/5KNqNbVx7+xsx7PZx5sUnceTkDUpyFEtVzC4eQnlyAk9+7mOYmN2L/Ueu02IfO3YUjz7wcUzuO4LOsICP/t1HUaMq8dZV9DKFJMkeGUU2asis04QdTmbVIl5HNebIjHunEarJ3ku1pcSQMTVoFY2aPDXX3c1ta4d7VYWS+4RMM1YjxYlnSMjvdz16i5F5P3rXFk7mVaX5rne+Gwf37hsldsLBJFeNY1LbixZPTjCba9i4naQQfk803+NX7sDwJaiGubhsTBC+C7/yOjqZIA1t0si9B6N0e3vHyCNk/uq4Spbx9pD664/8fjIzO6u2FWxNwSTG8ZPX4crFC1i7/CoOXH8bFucW8NzjX0B5eg6TlUnUG01cc/I00rkMnvvypzTA46ffpAXau/8AXnziATRrNRw59UbMLsxic2MLTz76EL789BksXb6sXWGevrMynMkSB4lG191oWZl4q0h+jhQqPgiPfeAujxYUVu/sPcZGoIsd8Cq1SJUfdc1OiJQqde+fAIXh60Md+CoMWiR9o/bypTiYcbP4vEAubQ1riO2Hz3H06FHccMONygqye1TUG/EZFNuzOW+vp13ISwVMSgRRi+LnpfCrteMsqgcMhZj1d1w0CZu34OTOpkIzSDnB7MysasXYnSoO4su62Uj99V/+j4TF6LWdOqqTVaxeXcbhoyewvbmGK2efw+yBa3H0+LV48ckvoj8E9u87iq3aNvYdOI7iRBlfffJzaOxs4/ANd6HEHT87iwuvPouNy69i7vAp7D98rR7wxScfwKByAB/72Mdw+fKyqb2BdTgO+0Xpj7CEoQapwnzIyLZx8Ny1Ukm0/Q5YyJN2gbFsmLXVjOI4LZYxHV6T16ZajyTQbjLFD5rLG7NVbBSP7y0c9DCR2kQcNW8G7zn3cNCII3CcLHZg/7SJsp1lwrCM5nHYbSmKoa9jdKs0+sMu7Y4EgYe55Qs2N9T/1g/V6r7Y+ULOGokjjZqKKNVpiTVfbPbXrKPJDlM6Xbfgba0HSP35n/5uwqpEa59cBM+Xmp1flId86ZXnUJpawPEbbsH5l55Rw/mFPYfEpZqc2YuFxUWce/ExbK1cxsTiMezZd1iLvXzxPNYvP4t0YQLX3vI2dSB89bkvoNnq4vMvLeP5xx8fqR9BmNHPVOwV271c5JKfFMDfaZFzu0kaIWV+Qq86D3i2R4APTxQKh8lLYwngMOHCtKrRjiyhEWaBqcoAddQtSr3COXF2hgfbVZl9NB+DZT8sMOQiqZuTzibxhgEOdFBQeF/ZVPfCC/kSDh44iONH9mNl+SoOHTupnnArK1dRmShhdfmiHK3DR67BytUVnXaYKxZVhdlt1sVJLzAbmStg2GubZnNIt1CqamytTgvVShkNP6lPWolz9Vd/9jtJvkxyoDVutzjVmrGtXDwnZujJG2/F8tIFbK0sY2ZxrwSjOr2gU/GuXjqLnaUzQLGKhYPXYnZ2Adubq1h69REMBykcOf1mdUQ899LjaO9sYjs7j4985K9Q11FN5pUyZOFXWtp9+/Yr3hYzxI8nZlTGn6lo1ZMz2l97VaaFFlSnFk7xWlJvcaY2QaOx46oihqeaFN3XF5+2UPdxhzHUvFKq7jCypo0aYZzUEeDLOFizGzNb7xQV5jmGoNjeyZgEnt56772YmpyS8DY2LmNicg7XnLwJly+fxc76KvYcPIyt1VVkEx4ydxUz+49jbn4R68vn0ajtoFouQIfjFLhBymh3Gug0a+i1TdAIdnE+Un/xJ/8lId+Z+LUC+X5f9pDhQH19BcNUGvsOn1B/tPUrl5EpltUMNpUpYe/ePdhYX8ba2efFtZo7eB0W9hzAsN/Buee/qCMo9p28HYcOn8CVSy9j+/IZJOVF/PnH78eFM+fQ7Rnezfvu3bcfh09ci/m5eeRy1sEvuv30O9bnrMQDYZx2LBXrP3Px5HQZqXrk8Qu8oPCy+I5xrjea5zPy89FFOECX8URKNKoNgYmkCSnBStHGkY9RPDiWw+Z4IlY3xGs3JByhdrLhPF/T4F8ybCmQxw7OYX7vIdz9unuwvrKEKxfPYe+hw6htbKDb3NKc7T16E0rVKVw5/zLQazGzquKLfGUGM/OL2NlclZlg10rejzSpEos1//T3fzkR31nF3XYqnzrRF/LoNJuC6fbsPyJbsaZMFoeWRbZYxsL8HkFzK+eeV0gxufcYFvcfE3l96dXHsbO5ganFAzh6/BbU6ptYeuUZtb185lIT93/606jvbKDR6eOHfuKnUW8P0B9aX/B+t62meYwfCXiwebwWiIiR0CnGqhazdhjX09apM7E1j+VxVRFeqcpFaUMrciAwRE1g6VaDaMPTDR5XcMnioNnIkAmNU7WqMWIDsKHNpcPJ8NLOFfXTdrx8KFp18/ddnnnqfcfl7XtmXGeSqZdMTxSmQwcP4Z7X3Yna5oaAm15vRwvOse+95laZ3NrmEmqbV9H1as7yzF6kszwQponWzgpSgz62eYpvZRKTc3uQ+uPf+/kknS2gQM/RWQ18eC5Kp832WAkmpxcUpNNpo//KTZUrTmDf3gMCA66cfQHDfhPpyjwOHL4OxXwJaxdfwtrVcyhOT+PaU2/ULl8+/6zUYbtyBL/727+NlbU1fNcP/LjKaLa260ilzYwQwKF3WSa/LUlEqqCw8RpimGZJY2L/MaYQ+xh2efRCH722N9cbU8uWGrXr2kIbYNwmsqdG+EaJChiWX62Az1pYRIYvgI02QxgnSQaiJWqSw7KMcdXbTYV90aXJEiZ23rbF/vZ9HMhqHRSkPVRTwTH1UC0V8N6vvw95HajXQnNnW4zUvcdulTlbXzmP+tZVdFtNadvS9B6Z1+3NDaBXw9ryZWvik6RQnV1E6g9/62cSNpnLuo1MeUaF8KBaMOoQlylkeUh3r42GmCZZtdCYmJyRyqfdbuysI5cvYe/hU4JXV69exOblV8XeYAjGU9uvnHse9Z1VzB64Dn/2N5/EiVM3Y3pxn45n1IEvLEFVKGPg/wghEzrURSGbt3M1szxkhXGmgShpgjE89LxnXYLZs7TXZN6YkGRXNdGKad37p9dPDRKN9tSvLE+wYjCCcFlxysW26CCl7gahBfg7zoslM6xsmDvbnD5r6MfFEA7gvcKjC4Oa0PF0AF7DY2p+r2ILfc5r5HrWFLA6kcc3vOPt6LcaGPa7SJcncOyaWzBIp7B+5Ry2rlxgcY5M4fzB61EqTmCYdFDbWMba1SWFqRSwyvQCUn/wwf+YkKhAiaItYvsIhhNsXqf2Dil6x1UZeXYopoqU9BdLKFen5KVurS+hV6/JBMzuP475hUX1DVu/8JIWYM+J27G4cABXzjyPVnML5YlpPLvcRXlmDp2etd8S89QXkhk224l+aqA7TMzMyXazl6p77oasWSUoEyqceDaHS3kbCi4YPVnZzYT/DeumqdFB65HedWKAWlzJy/YjLbwgYChTMlCOOrSAOYK77BtpAbD7RFvevPkJ1pGY17TkhrUXCdqQBMd9iPBfDDJmVScPaAW+5Rvfi/SgZ+ZtagYHDl6PHoZYv3IejbUr6LGWPJNBdeGYmgT3ei1sXL2IAR01xuoTFZSn5pD6g1/70YROGNtIkFrERVZK06sp1JvDKx0M+7W0W5LKYnJ6CplcEd1WDTsbqzqFoDp/AAcOHlEP1NXzz7PfFqb2X4vZvfuxvXYVm8vn1PZyYt9NuLTdwOb6ttAuJUl27LhFmgp77Ta5s7DL6sO5s4lghSMU5bWMyyWILhQcL71QCpESFd6ey0piTCtQGFhTpSMn/WgK4eXMoHmKUhAoETcJgZU80RsPx5Dawzh1LHw0UkR49LxnOHcBgYawBFrGnyk00gxjPVzlHWWzeM+9b0C1lLPqmvwk9h44KlOyevkVNLau2rNkM6jOHQZDO4ZrO5uX0anXrCd8Lo+JyWmk/tsvfH/CKgZCRTlWIFKUrNLLzqygM5GyKkURERkzisGWQ5GdFgoTGPSaaNW20Go0QCeBi02MdvX8CwoBJhaO4NCx42g2a1i9+AobV6By4HpcqvWwvr5lZaaqELWJ4iIrJednafG+ERLxIQmSiEbknCum9Pi5qNfm7jOWqhMTiaDpyGg7tkH88yGUk9fnlIywMLA7sG4S2ZQVshMjUNJDXYzICvW0qHvhhoFbXpq7qOskD2kYp2AFeV+dFb6mTCcSKiGMwaAJX4Ff3/2W12P/4qzWZXrxKKbmFiVcq5dfRae2au23CnlMzh9BuWTtvzdWz4JUETmZ6Swq0zNIfeg/fXcigqHjyAmbzbK7AltLyzYzCc4qA3c2VFCQIJPn+ZhF2XpOXmN7045xqlaxsO+ornHlwsvoNtaQKc7iwPEbJCjrV86i3+mjtHgMm/2iuFRXr1wxRMhPD7BeXl0hZOEpR1ZMRx555YUQLSpELz5Uk9eoBGU9eJ4q11RmxOKWnuTCkCnCyfDzNpyDprM0WJbkvdA73ThegpSfFnLUbqQww05D4PUUQXS6fta3lSSHLQ8nLnZ34O2RJo0jKFyVuYDasVFxxOV77nsD9sxO6muDMwAAIABJREFUSkUX5w5g3+IBLeLm1bOobSxZGXRviPk9R1GZmsH21ibQ21I0pANwGx39PvVbP/sd1AFyoDgwNokXu8MdDJaeplM5JDnLVVN9m9NCmnAJ7A+mZCNVx9YWUrk8Fg8eEzy4fPEVNLeuIElP4NgN7kEunUW31UV25iBa2WnVSa0sL2uRGA9zt6lGKTPEsD806JBN5ssT4IlEskHecC8otOwWQc+a0Kd2ijxj8uDN+7bOidYWK5L+dK7YYpMTpaSHs2aiSWyUNxGv5vENwx6dKPY86arUNpoXtPtdMw/eKIj4dajigIEjPx8xdhAX6DyFoxhCbQ1sR2WaEuy3vek2LXapNIGpfddgbnpBuYzNlbMYtLcUmRQmJjE1sx/FiSo67SZWll5B3rVVNlfEgIWHH/rAdyZiOaQtO5RmGwmiUZ6xIQKsGmVWJqZTVmzOXaiOPEWUJspuuwaob22LZTo9u4Dq3CK21y6jvrksFHnx0CmUKhWsXTmPZn0HufIc2qX9SkRs7WwpyU71yyOQAokKtRyn+ubyhosTdaKNJVOTqUL5QGOlM2Ez6UOojIZwqx+uqkn1BjTMGFEzWJ8XClZeuLLial88xqqETOkEqTmfU5iUVnXnyrxpO4SdziCzXJEAEVbujFad3R1HZYjM4Od8e8M6TmQc16gx+CE0//xdb0KF53snKew7dBIL83sl1Mvnn0ONNps59HQWE7P7VRde21lDNunIBxLUW5kStzD1X372OxOzOVb0zZBLaFTBHDX2CleaMLFQQkcTqNk5Y/Gy7IF1sx+q9zYHWChXMLfvIHrNbaxcflU2ZfHIDZiZWcT2+pL6irAJfXfqGvkKXGweDcFqTsbtUaHoLbSlVjmZhFE5JmLcUc9katGQNf7nwgX9iMQJ29nBJPXKEYV5u6fvMU896HfkeCrP7nGwbDeb1PJ0wFJeKBfrzsLDVt83liA7kKJkhjtYTGTQOYquhMYPYzLeqFfRwcJy7pGPtwaC8iGcEcr+qd/yjW9DliatWMb8PvO4eZrP1sqrqG+tWPuNdA5z+46qgrTZ2EK7tqbjP3QC4YB14hWkfutnvt11hpXQBhtEh6MzvFExALnZWaTzVn8sJiSTD7Tn5K3xZKC8nYqrcy1KE5if36sdtXb5FbFVJvccxszcgjr4s3mMSIvlEwpVOmxDUa/LuYlcbuDVlvWx8ETd/dkf1Q84CcZKwkXgJDsi1uq27TQgr57kLlVhuoTaGTHe2sPOv+buMz67cs6eCrW4Oiv8nCRJOX19rzrReR5RgUJBs8pSMkeiEQl3KtOl7CYch89F01i69jI3znc3X4MttqzDAgWHWmeyMoH3vO1OTFan0RoMcejoKVQmJrFT28L60lfR7zYFnKTSZWlT9UEb9pB0G1hauiRNUixPYDhII/WbP/2vTY37ohqldRdW1NmWKo/M0OCpFFUYsnho1geMks42URaCMITIozI5h8rkJJbOP492s4nKwkHMzC5qR+6sLVviYvpa9NgxMWV8rJ4X64fHysmXSiY1iBAn04I6e9MSGNwd3Fl0jnhdlsFGaSwFNc77oAqLuF2qUud/GeOFcTX/RuFmbRuJAqq58lBqBIl6fM2TiMPmmrnY7aYcp/Ba41w3LXQO++yVZJTrqLSMggdreGMLLSrx6IjqtDTD1FQV/8c736S5nZxbxNTsfoVXPDu7sXEJnXZNglyd2oPK7KLYNIxqCKrwpGSmr3fqdZRLk9zZ36Fi/MjcREDPiVD44+CCtX5iC1s/c1pnhDA+ZjuJtJrCMUHP9BxDNoIwk/ML2GKXgc01ZAtF7D10UiqPP7MNZmX/ddjqG57MhHuj6Uc9DW0RR6GKdiorTzpIuEu7hpUTEVP7KLbS9J7oXLxI6PBZomCdpkjtuHg3jdvqrWk+goIbTQLkoHq7jvGwyey9dX7UGVrcJN4dOUgQ/MoIYLz/anjaUZAoCpXrU+5sgwGN2B9IG1uAc17vufs0juxbtM2RLePwsetFaNje2cTm1XPotWqoN9uYXdiPdHZCm6DXb2NjdUmhqDUw4Jrlkfq1n/y/VJ8ttTFWlmq4MGucrMsfU53y1kX5zWHo3QJ1oEqprF1ON39re0tYNosGipOzysisLZ1DtlDC/P6junnS62Fnex2Ti4exmSygM+Ahbzy1hhMPdFpNLabSrCsrQsbUUbHfwvbahtSikKiehU089ti47XZS4Hi1pdGS/MSByIJleaotbbkVHhi4stulwPhscYCLV0+6lpFH7WQ/2d047H3sFEE7etF4YSE0VmCw26dVrFvaZTpq6pC4W8BHLcCzWk7fcho3nziMTqsmBK5QncUij+FImGhpY3PlPHrNGjvJoDqziInKnO7RaO6g19rRQQHUVKRIsX9b6hd+9F8RNbbzPoTC++GnnguWeo/KSTVbpUfMHizehsIPbGOF8GR1Uk1pq1PTlldOpTAzN4+rF8+jN+xg76HrpHImiadfWcLk7CLWM3tF9WFMScePue0aKTU6M2tTCRFmgsjk5RENje0dqXvBlElw2g1vHq9uDApSLLx2ZZza5+UycVipOh6JyMIODFGf6ScI+yLuxskegqrbgrFbuctD3ZN9kuJCC//uW6/vsb7qTGqIaDFioBikGqzVfDaDt977Nhw5ehS5BNjavKjsI9X9/IETmJyeQ2o4lBrfuHpOY6YWzZd4tGNFgkuKdrOxiWG3Y4fJcjMih9Sbbj2U3H76JuxZnEW5wGMgbGcYsmTHOUnL+JlVVNuSfB4xIftt8CV42MpE2equqxXtNDam3X/oEFaXltDpt7D/AFG0JiqTU9hcX0OhmMdw6jp0kBOjIzhZdNSIVtG2Moxpt5totWroNNtqkcm/G1drt8JDp+xSCBMoHAv4MXaptFLWIFYdqRB9x7UQdppwf2AkiqhBD7ttTiNtOyfDW2RFoTyv56Wz0jKEPcWMTsk5ox7ghomW21UeLyV2ib2OHz2Kd73rnTrakX7H8089La0wOTcrz7+2eRk7W5tqaLD/6CkU6FUnJG3WsL58Fjwsjru2VJkBUkZy5GIPBy0Mve1GVwfDVZC65YYDyc52DZ1uH3vnp7BvYdKci2Qg7teeuTmxKKpVghpMORpRwFgtwqasFbPjuJwoeucKHZIheEYlJW91dQULe/ag3e6iPDktQiL9vurCYaxiHgl3sLJUHaUtZZO7jFlbaDUbqO1s6G+M5UmOCOyZE0Shi1NpFaOn2bynjEabJTNZxc/WoZ+JClOlPG6AgsoiCNavjRIgsJpoU+27rUWCjCDVOxiiFGd48z00H96TLCNUz2JrhWR+AnAqm0elmMVEtYiDC3tx/fU36Pip8ClUxpMCnnj0EQlloVpFv9XC1tplgGeDF4ooLxwWKbRR20aztYN2bUtzRH8qW6yiVK7aCcHtJrrtJhKCQATApE2ySH3vv7o3YTqvR8eDXYa9+ZyqCr0/mb7qRAErLdGBLf2hFnl6ahJ79u7RQSqGaLGSgtUQrGe2Qv04TqJa5Yl5fRQqVSFOxL6LE5PoVo+h1UuBNWeKibsdLQ4dL8boGxtrGrg87xbP/zLcOcJEqWOPkYm4EeUSEZD1awXrrM+QjQfAqgyHKFjBCIUsT2ZhgEgDNGEeOAU3OxbZ4E1r0MvPTfL0PyJnLhhWnsPr28HqFMZKtYo98wuyvRN54hCb6LR64gIUJmZxww03jLo+EKmjKfvyF76AieokSpOTWuy15fNqbstoZ/bQtfrabtaxvrGiEJbRMdkz1akF7XpD69qq8GFYxnFIjdP3+vkf+iZtEjZmV6rNCXW0wZwk4b7qprRbtald5z1MlaPyqg4V+fnpPTOzM7j2uuvEqCAIYIOwDj4E7SNVqQashTkkU0f1WcbqFBR+JQOD8XOzuY1+u6OfyaYUB9pP9RXgIgDD2leJBOAn7vCe6YxVTPa7BF94CkBJlaOBgKnvJ59HqVbadfNfmC3Ty7NbnFUlJzy2Vh8G92tYp8Wdye4Kx48dU/NZ1p2RYXLoyDVoNxs498LjSPptEGsvTC6iNDGtkwXjUHoWPfL5udiV6pTCrPWVZdRWz9uclWew9+Bx45HvbIrlQ4iaY2r3eiiXp1Am7yCblT3vd5mOrqtdds6Zralf+YlvVehFhUz4Ubli5oVVAdGjhTJnw20UmV4CKFxN8fd2Gp1liSIG5c6k/TLbbwT9bsfO/5pfXJQ22L9/vzx3kh6Ge06LVkumZiQSqKLIrWq0ttDheZs847vZsF2tQ8GNzMAXcXsKJl+BSRND77Pdh0jypFsVBcwwNOFY5ZiNjk00Z288V82Ja+zU7JgI1rn5ATlk41II+PXUtdfhmmuuwebWGmZn5zAxUcX66jIaNfLF+rjx1rtECrx85ln0W3XNyfz+48gVyzh06JA0DL3xKGp89OGH1fF4Ye9BXL54Dq3NS1aDXZzGgaMnNY9rq8syZdnUAM1GU2dwZrLkBvoZpMOekk6N+rZiciat5KP815//ziSqIuwQUivoppo2NTeCeXczSqPOu+pY7b834ELagQkJP/vLSkkNmaOU8e+0pXSoKCjqMcJMenU/7nnft6Pf2UGjZWgWsd3hsCe8emdjw8kTLQmWtWvmrjWP02yxOZb8T4I+zzmhGTFP2QiJKrLzDglBPxpRguh3iOPmJ+QxqZKy9GppghqqjLfde69ds83zQbMoVytaTFasVqozow5Q3HV0Lq+/5Q70Wh1x6evbV6U5D5+4VZNPPjmdVDsdyMptv/DQQ5jU4Xd7sbWxgtrVc6i1apicP6bUMcda49mpTXaeaongQLw+V54VtVspzWSI7Y2r5tekmYqeMELGf/9F9kET3OMkPe/d4VxsoWVaLMNwhdCovYNpOU2hkhCEuaPO2tpRmJPDybfLqwGxeox6aa4awQzVpyWXTuPU130LtjpsoleX3SNEyd5xW5tb2FhdQTLoOH5uxEIuaqdDLNwiAnnebPQeDVr7xLG9/4rCoYHIlJEGDWhW2pr0q4nyqE6d5ufmm2/GwX3k0PdF0ZXjxRMH+fBeU85Qi1jC6soVHSBPUn5UuzS3N3HkhtO4dPY8Bt06NtcuCTy68dZ7sF3bxpEjR3RSImFTWhCO60uf/zymZuYwNbuIrY1VbC29it6wh5m9J7Bn7wHVfK1dPS+NOzs3g1aTMHMH+cqsauTps2ysr6K5sy56mBrv8Yhp+kh/8ts/4H3QbCFUye8Hh9mC+lGAYyfDKhRLeeMcnbgzVP438F1CjwJivGVlnE1l8pSo97ZMgxPuGPqo9CYzgeqJN2qhGVq0CBgM+qpDI6mOtCjmzDfW1zA7M6NDaKKihF2XVP/k7TEMJCGyV1S8ywklXYgPTRvLF0/lLZQKKGSyuPGGG/Du9/4LhXWdTl0EfkPlGBV0lQ3kiwwcqnU+Kz1fmbp0GitLlzC7Z49OGZC6L2Rx9cJFXHPtdVheXkKqR422g6Tfwb6jp2RCWFBRLtuYTY0n+MKDn8P0zCIq07No19ewdO6ryoQdPH6bPPJOc0sHwHaHwPTstNLK/V4TufIMZmfmNa619avi3ak8macPq8Chi9SHf+dHRottIZf3J1HHwziT2k5mGLEhBe0ZnCreGp0kPyhUjEo/RMXAA5oDU+8Ww6Z1noaYrN7OcgSqDFNo5efQyS+g2W6g120pxqYd7zQaaDV3pKZ6ZL2y1kq4vbVfZm7aTtyzXR4ghQANP6ScEOTMzDTWV1clnG99y73Yu3efaYheG7fd9WbVk3OxL1+8LEHrdpog/6xcrSppEW1G5Cc455sTWd/awMziohaRqrY6VcXls2ex//BhrKxela/BoorlC6+iunAIczPzYHRSqfD4KFPj1C5c7AOHjomHT01QX19Gq0Ou+M2YmZ7FkjgCqyhVyRGfx/bGhnh9E9N7MDU5q8UmgsYTkzkHC3v3iU7FRj+pD3/oRxPtwniZiR21QTYQwc/zEp4ah5fa7uBLB6V6laPgVe+sFDndKGS3YwYtAxSokmBFaQ1ChoYuDZmTTU1iY7OJrfqmKE47m+tsrYB2py6An+8jt9zgyzTyaibIrhAFUW/Z8oKeN5242s46zp05o5OD5YB5XzPrMgS0egNcunwF/+67vwf33PMmdfl/5pmnMTc9qaggSn051kbdNAjPqpYvkIJUJ/GAyWpVOALHUSpTnW5gbnYaV5eXsdNo4Prrr7fvazu4/ba7jSY9wR7ljAKsCPHBBx/EqVM3YG1tXdy+2uaqophD192qg1fPnXkG2QSY2seESB61zW3UN1cxtecgZqbnVQ1y9fIl60RZLBnbKE50+JPf/qEkCgREY/VWjdEPk7syXsJ5/Sxt6/tlQqKe2+y0pNaNFAw/US96aXpvci66drtfUI4Z0SQ/F5rHJUl4vM3ygWtuxeKho3j2madw4eISVq5exZXlS3Lc1Bd1dhYnr70OxWwa1UpJMXJc3zh4ea8qoZcgN13OA3ciNYQa1w/TaPUH+PgnPoFbbrkD//7934/6zjr+/u8/gce+8iVzbPw4BjmTxKjzBfHv6E2fOHlCLBoVEKiYzzooMKTiTQnt8kU0jZWdWyR4qClRWTa7Up2wolB30D73uc/h5MnrsHR5SVU4w14T/e4A+07cjG69jo218/IbZvYfFBeP8DFbWk/M7cXePQews7OB2tam5fRlwzkHnpn72z/8aanxAOwjTKKaVk9MERVYrWidjvRSQsEWNGykcrFjjdnMsTPnbVxpWBtn7zzgxxf1ujxxqCTkSCfg+HX3n7wVB/YfRKu2jVy5irnFPejq8BlDuRhFMDR76cmnlOyQifAyXFtb4/AG6udDdxKenxDkDNLBMAfCive9412oba7ghWeexSuvvjRKDgk1pBZKLEMXzeLJsKEfEXRg3mNyakr2mKElNYyYs/W6wkzGv9RGrVYPr3vDG9SEiLmJhKnWYYJHHn3UBHYwRLtZUyODZquDI8euxfLlC+g2a3JoF/fvw8b6ppVZnz+Lyfm9mJmdx9raFW2GcnXaDnuX752oKDD18T/9Oc96xaLEQRu2IHTVY+G4+GKMyMZ46exoMQ0UiMW1isZd+dC1YrZdnYcNZ77ZeG86ZXOUATp43e2YmZlDu76NVg+45uRJk3T2YvF66VaziacfeUSTZbVc5L7HgY8mbAGt8jMqDBiZJdvsSln2SKIs4u4336MzPK5cvIiVlSVD8lhPXSAtyzo5jkwQixG8S6OlVXkd4tI0N9ZhgYJAweDPtPkkVcq5K07ge97/flxz5JhCKAI/HOcjX3kEO7UaSjyLs93E1GRF9fB0tLrNBiaKOVXDTs/PY3V1HYcPH8aV82dQnl4Qf2Dl6iWU8gVx0phfiDPAei0u9of/s+9sSyJwN5jjZd0LvARaDlks+rhaJy4rmk5sei/U293NVNbet2t0wIqfejvWEE622lmgUTZz9NQd4kqz9HRzcxu33nan6EN9LwgkiEsy4PNPPAHjjscZnS6oLm3xe9M+u2duywt2fjzbhPLnm+5+HTavXMH66gq2ttcFCAlhcx5ZtJuyyfImc+54RuPa2OWMAthjbhxyVeTC1hq9Pk6dvg33ft3XabcGBflXf/VXsb25hTvvuh0zs9PSIoRl2W2KHZwD++dYGT9rnaghU8DUzDQ2NjbF0WPju+iwVC6woH8LqU/+5S9rZ4fKDRUbReheyTc6fZ04ehh9U6XehMa98dHnojmNfm9N9ETrkZ0mxkwN63XVbvt1cLiK3kzLnLjpbhRLRXD38nD1O+96I5JhV8QH+ges/OA1n+VikxDo6dlx8zFuRsxRsVMLOOlW62VsWXK3KLQ33nU31i9dxubGGhrNbSUQQiEpDeu9xSJEDWaqJYeM/x5HJGqR3dkN4CoqRukLTc0v4r63fb2gz26jJkH8h099SpwAopTtVlPPvr29uUtXJmihA+ZSgqzvu+8+1Ld3UCiXlG2k+aht76hogI6q2Dre/Sn16b/6oGlXV8dsnRFVhoq7YWCFuFGOhu2abtsZHCQJDeEcGcgSoIqlEE2VxiEzpt9JXrTT4Omhs5uQdxvy9OO1N98tpIxNbzc2d3DrbXcDSR+dtpEWCMgQwHjpxedEpzWYNHaupSo5vjixwMa/Cxrp++iE3DcTdPr1r8fy+fOqH6cTx6DTHDM7mUDM20gWceGdzCAz5R0gomOSiIuuScRC8ffaGEijmcBb3v4eVXU0t9Z03ccefxy1Rt2Yq85eVX23OkuRjGnnoZHvTu4AfQGdlUrT0TUYuNu2UwtOnDgpp3Bxcd5qyD71l7+h0Mt2HA8xsSZpRKFMPXtxwKhPib1P6tDroQlUkJkSXXCDdWEPz2YzfmqdN3qLUMwOHkvbGWx8qQGvgTH8/ckb7/TzNbjYNdxy613I8HRf2h9fbGLNr778guwcXxEh0GdQBYvzxU2VjqnwMSxAdeCevrrlDW/A0pkzKmC0fqm77bkoKrTB6tbsr3EUTjZ9LFctyFjQoh3hZEJj41AkkCvjbe94L7r1DWytXpEwPPfC83aWp1pVG8AVTXEZbYRGMg1h1SnBqOUCc/HJ3AmyhX5uNc0p/cSf/1qiRQ1P2rsKEQZUJkdlMFbgZ573bvM3O/PKbqgDUehgSQ17LjgcNnfOwlFidkgagR2FoxhdYZA5TKQv8+up03eKSUpEbWNzE7fe8Tqp0XZzZ+R4MYw69+orst100kYayk/dNQKGTdiIheI2llpD75fmsTHfcMeduHzuDJo7NU0QkS2xXvzc6+C0x7OEBov7aq60820xdGBtHGrLa7Cu24PP3jCNe97xbgyaTWxcPa/fsuecAVCR0DGuqti23lvNSpssK2lA0mudYwaaIm26r0HsXJnLB//+vxso6lAmOwT7Jhsttv4uAiJ3+lj7Z1eJRtAzMMVjldFiCK/2npzhrTOjxsEqc+axLwWHfULMKzfu+nU33+HYb1uY8Onb7lSIxpZdro+lwi6cPydIlU6aqVNbHMX10VB+jEQYioQecoSOAfjceNedWDpzFvWdHfMxvADBivt3SUu249wshB13tW6pYkvnkshh2IVrQ/YRVTjIurIEb/7692ix15bPSdjOnLHjLWNnhjDp7G3vrhRahfehWuecGF/d2EVc7DA7ETnIdHzm47+XMDgfSv34PyfmaZF0UhzPf/RmMxa4CfHSronuAj6ZvImdOGelqqPJVAdfO+A1doEWX9CrxMkaqovsZ6f63va6N2Nnh2yMLlbX1rD/4GEcPHgE7caO4mpRfns9XL50CVubm+Kgx3LwOgQ4RlI/5liJTOiHoclPdDVObXP9LTdj+dJlMWnIXo0+M+HHBIEhTvIbuWxxGq6r6NGCeZM+Cz0t2WSwM88USeMt73gPeu021pfOCjc4f+6MLbZ7/+FjKKtHAfFW3LbBDGJVqYo2kB9O5+FmNCaK45hTn/rb31EMUSyzH7j5nYb5+jmY0TpSYZLtCd5InQ7Ey7JSHCMKGL2YixkQbOw07QS/VrAzQ3p1Yg6rJxw2NcnN4vSdr8fm5roQI+5sxuF33/1GtOm5wjQQr7G8dEU7W2fZOu891DMfSrsjcHkXKIVSLqD8W4BJR05cg621DaytXFFPEiFRHFsY9TFnVnVZrloDHYxdZ6cGBbRsjeN3Y347S6SHDO5953vEe1+7fEaLfe7Mq4rVJf5+T/lI1ppAOL11d6TZMc0YZA3RrLxvfKzVa6KRz/7D7wsuDXqNUYqNVmyOWCBj9tCjzkTqG8qdGylOs7k6scZzmrb7DR5VViv8Al8AMUIlheYV6+jBqCbVzn4TVtdW1FNlbXUV3d4Q97zlbei22KbROvJz0VZXVnHl8mVRbCOc0iLpQBpXoe4oUXeF+jaBsNEJ8k2l0Wy38cd/9Ee4++7bsY+JDR8bif969miU4/6KnWoQjFwzcdG3xZJAMbN+JFMQHYnLI4Ove8f7MOh2sXLpqxLKC+fOGiHSVf04UBU5i5G/4AUOfA+F3tg2u5z34BGYtkwj9bl//OPXhF6jvp8uwRZnGjFg1NGXUpqN8yzNSVMxgSNmYZ/ouQZyZuc8ewStE+fNhpla2z1wLVpPJEkGt73uDeKNE3VaW1tDu9XHvfe9HT0S6nqsDrHFXt/YwJWLl1R/TafFMl9GJjTeuFdwqurFgJAwLyNAiAxTb8BnThaBlK44dYahu332tG8cZ2k70M/T8uOVAjnUCX0yJxae2nvjUBrqoQze+Pb3Ydjt4erFl2VzL104PypTskNndzsvhUmKbBvVeFCYAwCIsNds9Wtp0akHPv3HCZvEcbEikRF2wj5odjeAjlGHP8XGpto5SOFkyrCYBiDqFUcbSfKVMTMzoZN6vM5bu+s1xQnWYJZlwjfedieuXFkSAZF9vtge+g1vfosQNMba8fCbW1u4dO78qLOhjd+gzXhZZskmWlThcC69gI4cPOLyjCgsRy0RN36dkn3m8UYyJeLqEOZY9N1FlTfgHrlpDyvCsMZ4pC7TQXvj13Nn97B66ava0ctXlrxvmrFr4npxX9G8YiMyeRKaw9GeCNMsNIOyfqbKE6Q+88n/mZi63T2OgWzQkPgIAeiI6Wxt503HJNruND0tD9CPNLJF9ERJADY6dshaPlscGWrcvGe1+VANOFROdN0Nt+DKlcsiGjJe5K3uuvtNKp9ts10jGZnDIXY2t7C0tKTF3t0NnJTdHSV17tWRHKfxvmynh1Dy93TqZA+9twq/l9fL8NLHGyf0CGuIvqD+jCYg9j9UXYAsdhSym0hWtaQzeP1b3y2zd/XCS3LKrl694nQwW2gzpbsHxIiE4EWAHOO42tZ9RjlFrzVztFBj/cw//BFnWotkDEmLcUOiaHPU6DVtao7F+uqsMmYDxxeetczRRYg2kLHsru0O6lOoNNMXcRC7YlI/gJ1O2613vh6XLp5XcbmOccxkcdfdb7Z+afXaCPAgAHLxwsXRafajSXK0xjQNPK7AAAAgAElEQVSvh0puasxb9zg7doUgVMMR5Pw4SCP8OfBvPytr5MCS+KB22t5wncczSSgClTQCR+z8kXBwsQG84b73Soiunrf4+tKli6MTl0zQrKCB9xcnnKiemxRGH6G2Y6FDsEJj8hoSCP578B8/nNhxjP7gzh6hNx8XEgDiKpHzF2dHMakfGoEDVmd890AD4YrEF+fT4j+2prSzSEjmkzepigqj5cSk5PMl3HT6Nly8eAbNWl0IGXfg9TfdgcpkVa24wtPk37mzFYo4C3bX8x1pcn0TDiHVdnw+nMj4uxweXyA70NVACk+YasxU9zIjDIc8XtdZ2wolY0fSNHT8aAr7tKAdJX2ETeL1971P110+94IW++LF82aHw79RGOzZRvWIsYPkLTHz2ub7Sj2PHEKzmnHagFDSz//TR/ycdPPiVJ3IAckxsA5CmhTufH719GE81CiTNLbIeix3vJi14e6WpvAMWZgIo0BZmYyFDLsxOG32DTedxoWLBDi27RhmAi8Ts7jpphuxvbkyMjU8Punc2bPujVvYGBy0sFcGUY6Lnjkv2oVj7SflTwgxtL9FoY5Br6aZI4YOkmOobd4rMoYyYd7VP7xyhXBuhzWSYYJjN9yJ+YUFLJ99XkJx6dIFT8zsEkkS1xaMDKKq1Ha9JX9Cc4+bFX3v8xtRTurBf/qI5mA8WcBBy5UXROdsEpEIqZbd4Pvp8qPdYS6It0o2BIfgCr/GGV0kPASiEzF2TJCpmzghwHb88eMnFFY98MBnMD8zrf7m7V4a3/QvvxU7G1clkRScdqOJJ554VIsklE/OmSNebqujowHllTnvXZ/EBCBsXxAwKBzWsM6OUQqKFT+vfi2+ix3NlyCrSCKQNkcIzY8wGrOcRO+faioshfmD1+DosWuwfJYdKmpYY6gpLWKJFUszO1FEWDjPzbYiC/V1k7Aa0STmdmS7vcFQYA2pLz34vxJzauyhTUpt0qRu2GBdyQlzZlQ3xPeN8dQIpqhk1h0fE9rd3t4SHnVGcI/WVVnYwlDdcX/aTd6/1ezgwsWLytpkSK0Z9lBvDfHP3vcvtLPpuHCR2IjvySfI8DAVqSOYvSWnhMpNk7xgn6jY/fKmvdWlhWzWuzvUfbBrHdUd/T52EcMqdV3gSSd8U2g+PxMkujSquTZbcuq4rOixDmTKU7iLIea5M1psljqNvH47RNPGz8+Lym3FDPaKGF5++2ixw2FmOXAwSCTsX37of8lmW7Yodl4U5zP+cFBE9un/a+vanuuurvM+siXLsrk4zTMdGAghJc0Y22BjoLSZ5rl56kuf+tfkodP/oy+ZydBppkmAkkkoNrbBKdB2aOMB27JsS7Isy/iiy+l8t73XUdEM2JaOfpe9117Xb31LXYzxtLvTwR4pSR9LgEZeVpvIk5QJtIYnSxJVoAiPCgRAGTpVePBnQizc79H2pJ1+/e32zb11xtpsf3n8qF358ss+WSdIVpLteGFyvWrBs9Gx1QzLEJWYoCejJ1QnF0gDa19LpQHqjKhFJoxQa288TyHYI0pGTcI0abtzi+3Ea6+3m1f+pz14uNlu375pG68hOVhPcdqonJo1wXvt0kGTyQ1zlMRifHEtAgP/+MN3kgrhZuGHkB580V4nVu2D1nSxWD8qy8zI1O53tZh/opU2C0nPO2AFfxbJfKjG/Sc8JkA8prHvc+2Vk2dZDHn0OM342+3alSs97MgIKJ7ylAvLCU6uoJuqMgVQalnjmkZYpU2W5jGO3oyI1GY9RamedAnPKBgBlgQAYrQBrquDMNd2JofaqTNvtLWrVwiWYHrYqNVoGBZhzHmukM5OngfohMUh19f+qCAUT57ZynO/+wWRKnFociFCiJ3qRFYLtyAQwOq8k7LtG8fESlBX4QYt2u6nt5kSywXWwpBxCKrTIAeeOEnQjG1VgmeunX7zr1gQQC8TrgPM981ry4ImdfuVCYBKZgw5hC0WsIGLY3oLLbBKrqlmqZ/NiFW/p+RTAh5SWaP6ugaqmwpsu/7tqlfSpTxYmKh+qJ149S0WQkDTvbGx3hEv40gNkASzcp6AoEepYazVuvMe3XYnawc1HrTJCFdU4406pdfZbbRjYdNAUkpt63Pao0T4kvbMueIGFqpBXYstG2SmJicpFFZgrPAAMOq99FyvvfmXpKcAVQe5UnYet6t/RNVoh/9WGFeRMlrsLB7Xx+YJz8AowA9dVTun7iH37Rx6pgNFjQOmS7gV/BHWA3TiVD8Y3j7u1zeIc7vAMgVth3U92E6++jaZHzfvrfNkax9k4uJYZk1xVX6vqGrlPGBf5LDFXPR7JtV7/sN/0TmK+q07ZueAC+1eLv1dthsnAMNJ1K9tUJ5TlXJsaj6nPJ3Zi4C9Vi+YHERsR8hnnLB3rK/TFOfxe6Cu/s53ScRD4va97bb89dV27x7w5KMql7q2RiaBv7Q8g/8aAVdoOODFiU6kqFyT90LSJynwJPoeJUfOjeiD2uwxO2Wp0Y3yReDRo8x55s2ftDsr19rdzVX2d3HsYuaTs4xc0rV9/Sv2L1UwPKfEQLG6BtoEmzf5+KNfWhvY1ibD5FOZE231L3XI/8+Rfjqgh8R0OhlyukAGD3uM6TScqxVbvSdmhJKnV8HERQeGPSyJJvGhaBfCxbz1wlI7eeo1MiHTmWq7beXqdQLzMk1eWkm7O4odKXJhBomotjnAVKatV+jkUIVpSAyPFMbAjqzNkkJNbE2CeY+TyGQAMjoZuqy5W/DEVeAgwufAQjvz5l+3zdvLbXVtpd0Bu7OdUzw7ng8jq6kNSvGoh4LVfyrIWWpVb3YO8uTiuV8RSox4MN7zrPxLavIL6c5E7hoLMsKA2d9KzMffcy4XQkfaSrSpGqCYe8bOzXrII3VL5KYF6e79x+3tH/+EuC1K8nSPNB5Qgdg2fTYmQCpdXrQ96V6lEkVHHDloCWgBYMz43LGHnPGl9ClOTNS3snWKh5FnZ77dzh7Sy2Ql3tPAG8wCwbVFSARPQA4UNvPlk2fb1vptjuVYX7vFe0k51CaMsgeZQNBDMK19F+p9Cgx97TzhF8//2o19Q8fFfZcS1qnqm20Ok3SI7BcQCcDYJHrDO2itfaiGOzaGuz2ocJbgaSAAsy+pxj1+z2kSXH9j61F78y9+3DZuL8s32ttt6+vrbR1jLayZ9LzJHThvwFh40Fv2iCK8KHZ8sAEsBvnm2EBQhuTa+X719mkryc6gUcbpfcv6wCuI40n8gEGIWOOXT73RtlZvtdXby+3uxpr6203Bid8H71miADwLINQcBxFHLQ0Y2WQntKANuHbOo0w+Pvcr48a1oYq2ZSP6ifZb4nvzC0JW5gTq1CTcGDavxsg4DVBlcsaCWvUm2rusmiD935BUeLOS2O5Cte2duXbi1TNtA6dgD1TVjQD61bVbXaYZYbg2YQnqJ7UKKN5JVJcgBhCsadaxlKgpdBTIQYKZcq4SStKOEh/6AbbjIBzQ9TAZQAT5aYHSlaft+6+cbvfvrLW1G1fbPYApe11cCS4Wh+y0Yj16+jNxvN86BzJ/ZjGgzum/fPrJ+/TGe87XKiRqNb8QFYV226ouqtrdpz1mBCI2T+p1oCFHBDAECCafaUerUiRzmFjh3E7QcB1qr5w63TbXV0lnhc1GVeyOwxY9B3qzTBvhWLg/X46odsZwXyWElFoc5EGs1ZcCDXVdSrbOlxPznjCOZV4lQsgOYZydfADhzxi5USUJRPjD195o32zcabevf9XubK5zs3ELMkfVAbR+NojIE08cJeKOJU+/x7etP01BiAAvXvgNN5ujkKIyi0cH0Bq+hG5UjRpf8H2wAbFR+3PN/Ey3s2Mel2J6PVbCL17fTkw2qsezOiszNeLJ3lw7ceYNOmRomwEVFurda+urM2FXMnYUqHjLAe7vW5nkxvPtekq0L9Ze7DEDoTxoLsBtLt61aB8mobxW1G5GfDLxEu44ok1R25cX/4MfneD1bl77st0hnQgcOCFMD3pONvYmpLYH5kWwHy2SZ0a/WOJ/ijsPixIstNkXzv96mrSe0p0eG8GN1WXYQOAZzIEWIc/dL+i71RM/CgujlDjgsb6uM3bJPwe5mQpVct2Kaw2AJHFKa6+cPkuqRoyMPAjH78GDtrJyvTtMqqPbZsXw+zlzOpMAyp8Jl7KIPZal0+I0qHMC1BzklgFJkNPNwIQDaMdcuzppoImY2vSJls4ZAEccoOdefJk+wvWv/ov1akQ2nLyEWjbsL4afu0NEiS3BrWhanOaWMI5iiEJJ5eO7N/7Jxfd6R8jMD913NfqmZgvwcLoYI6ePiDnzCnbDyRWqcn96tGqB5Md1kmvHpU5zCHPTXMeOyvmF9uLLJ4hU2drc4MlGFm7l5o2OF0tdW0I3SADY2xVOb6NjcjK6SQkg0smLaAVqtzQxWoDU8eFChVU5N3TG+ZTDJg2pJoqOI2tz7cixYxza9tX//ne7ufw1JxbSbNmHSpIIDpmG2TSSDsATUIg6Uqj0j+LQGrZMDBCe8dNL70+hluSAqBdbR9Y+kRMgWNioA0gKOwVdyYEdQsNfWlajgns4ZUjTQFoWtegFzKbIRimRoahN4Q2+xEwoTTO/+FT7/kvfaxvra+yUQBsQ+LWHRrFtdMIoaVTxgkeQMJoYU4+GY1nbd6qmx6IKqKiig/B64z26AHf1OTQaPoj2KHGrylZn+Pt0Z9ouf/FF+5uf/rTduHalXfz9b9t3jj3J+QfJjDG9y5aoxmgGIEgWeTxsjvjBRDhss7b/Yx9BDt+0Tf5w+QPS1ygLlLgl+12a9N0JghoqnAJwimUze2xpG8GUnoefiUZaeCxtYkIi60Z6uqlj25O1vOm6Dv8ywdaFvftb2+21s2fb2q3raqnZ2WnLN67xwYW8CdiwJhZ1/yAyldQaoEQKMdWkCzelb6tv/AgKVE0y5EfCaEfSCy7BVP9XNXFxqOqTra7ebh988G/t5PGX2xLYEiDkOLEGIdAEGlARcGgQrorHkdUDH5oig9Tgtd6mOMPJ5oPkQlalLKCzJQeDxlE8iJ2NLRinI7ZbiyeV5nRy/xMbqhYVLXYqO/SwS3IAzxLkClUZF1D57uScITo725N2/NSr7fbNa4T34HpQ4xAOaJioZIQq1AxpKS7v5yBToQz5VTCkVJuTtJqyqCqQpA5dHUuxUth/KSldLHFKwqoejnC2JksYpcB32d0207JnDXAtlQxi+AZ1jfEW2zucQwZoFt6LnSPBCYDwxxXL6lDOL5joCKFXjZmT1sTi4SEB36WtsXTizxj8bEZ+P6FSTz06hNCNh6qUDRd0SDEkXtQUlS6Q8HeceZMwZdYXBEA/Ovn6W+3m8lVgSLlRt26taHE8CObbMoI5BTFVaEmqz68WWzk2KnP63YkBB4/aYqfPBOYMX0ySlNJjDVsxIE8lysIeGJw8b6TcNZJO0n6D37xGBLTNHALPxXArspklQDO2s0NOuHtb95iKZqOCexnhXzFE+8OnH/Bk9w2HNDlbJVumJvpsthIk+jyrRQnF0ozmPHPQL0mpjkoQZosM1TnrIOhfeDC8PPovgi6hSvToIjiNsIEnz7xF/jEAnHEfqPEsdGL5qPP4EdFYET5ojapOa7go10WFGt6fm6PWpkQuNDJOzECFIudO79ydKGSz8xcFLSFpcQiUANq24zjajqMxs+manKCnjXCR/RkEufb6EYKCkpSQMnKrqYjDeWXZbJbnAhEuD8JeLmdw6oZn07PxgiHLaWHzuGdcRp0GKEBuEoP60BbcwwID6HU9WbugJ9FZwhAE6plqEz+bbz9CL9gaxkI+pucKB024OYdp6QFmbV5NinjAePhpeNMzJKmihnvNDpFGUZSQaESCykDHTfrcLJxId7pogfU93Pewiz5xDHNAcmDI6eJ5nMPZt0BZ02WdsjXSXhJysTS5X85FFDhyqk62Ptpicuniu+JUsXwn5qZnTika5bO8XCQuajwbSu1g+yhbaT0SRKUXVQkUdW0yBjX0iPAbniAFD5wGCRI3jIYKRNdcIWgP+sGfnyAPORiI8LV8Q0R1GuCq6hKEjjPLYJON6aID4znaCZ34bwq7bDcWcjbRkky6kiEJtxiuWhBjfxlaudFR3Z9qicY6UXNgpMbhxe608eCkJ67jzmd5YeL8cfMOmDQXc1p69+hen9pbBQN/R6jKwfCXPv5N3qKoKpXWuHnGnOUEx7mQsyUvOw5RVB3SfLAb8sQ1mTYmS6xC4u5OD1QnZvP1gv4Erhz8pVWNcnQkVOP0QHvm+Re4qWBTwtfNWyukn6A3ySxWAAvyVtP7VHFawZlhpHIydTpxo5iT5E5MQ9VG4CvXe48qm0yiT5WRPemw7KwUtuOBQDEK4LFOAqn4OEVtx9xWf6mPniZ0GcIoAYxGpq2HULDEabWU2LFWpTicmV8KnZhata2m09BbXUZlDJ/FaKI0ApL7k4wOJTwxL3naUxcwjQf5ZJ9u3BEErBpBLCRIQiqGRm2+PfEn323PPvccqSTxhRInrscMAMD729tkG8LG0dPmu3gRDaiP/dVwtREbd3SttRP+LSEbBQ8+OzabuYKR/lVUEpNh6k5DruCvJFNY07Cxw0Go5ARjU+P9x//JhufgAcwoBy5Jd534oZm0T5MLH/0rq1483oVdIBs/c+xl2fqm8WYHNMwktQWcZHCNcpSEpYs5Yo5zkMqW4GhhUapDe5EqOQbtO5QJCyEhSsjWOXTDS2AMIRrjTp89S55OfA+c33BQOILJbI1KWcqRxL2hbSKgSiIp0zcSOXIKs8AAEEbFwjT1EK33sMthGrWV8W69JOq05nAexeeuTXOiaF9KF9eMNoWwc/18GPJs+TlOblXz6XaJj9A10acX3p0KYTEQFUmu0AmxPY8nrGFPQwTojZY4mZOBZtKecnIY6/qUZL7IiKPtnTvMgfCgiiU7rWIB1ZDVssp9ILcDWO9UW13RlN6Nu6tkEEJ2j+zDYPhzxSxISy2iMk4anrrN7s2kN9PrhQWiEBotk/KmzMFgYooDV52umLeo/ZiebDYrab16WMD9xdPucbK/V0NevAM2P/kJYO/w/ELhylzVCCsagDabF+bpHl2JSONFv4v1aFRRdDId4xkpCjyV0psD6Ie/0zFQykhT64o9g4MWPDeegW4ZhrK5vpzSphZ+FDUEPFTv2Cuvnmkr167y5e5uronczYkdqjE3K8ZZVNyMcBJOHGrSek+ke/GFgkpMC+7BU4TnOuAikWktYeOl9r35hjhp2BycOxs/x+3MetnJ1MFBfludKTBP7Et3eKf9MG0XES0DRcRN5vQDHM5RtIr2JC22U8JB4cSBnpz78JeKswtTLz3yvZEZktrTw0hy8AAOLQy3ibSl8Wx42cp88TTCMwTkx4uEFRmqBpkSXR+4NQmF79VhROJbSYQA7rXjp063G1e/5qJt3d8gYgVCxdKsNUV6oiPhym0btEBEKhZdqBipSxHQJ2rgOAr3VGX+p5Aoo3Ajpw68brovpBFrgPdmehmzxgszFKpcMS34LBNYKSfjul1/SqBSWuY77Gl2N67fSXNc3NFUxZiWcXhpsy9+/B6LnWH94xksqqOnMp33jqOGFB4+BqaeWdugGVgKbVBnvt+WOO9aJzfM/iwPTveYhMClU8+G972I4kSHEkNbiJlQEjq0x/bOtJ0+c7bdurHMzQH98vr6Gm12TwyRqQnZJRHEQjUne8dqUkh7Jgca5lknjGKumc6oHDe0KjOGR1vSA00TTn93PO+0HkOYMVtLGyikqPyA0e0Slatr6oTCvMmpVVwvhKlgVPiKiYRgwy/Suks4a7TUEy5WL9xoCEnd7NjQ/FCGXW4lZAWSGbUGT5eDUuz49MDeN8DpTBtwVEzKopmDOUhwR4GCqp+w370+sD2AgIAIEepx8+cW2osv/Vm7uyZ2QHCRX7++zDHInNG5s026aPGaisRWeX45atgcYsvIqCBHM0PQsanyDVwx8nShhGVDaOVgIfqginU+H825+uwBhoP4PLBkAQlkrSEQ2fCUhKN2c/BynWQy8X1om5rBjOfdVbYrez22Z+jFk63TkpvGkajA9rSuYlIffh7JlIqEIKiYEs8RN+8xcWcDVp4Ym4CXxwMDyYm5GrhGkitwsLiAbmLTiXHNuKMolZR55pnnid7cxcjG7Yft9q1bYmBIWLgLFWlqjU5eo9HJQXsQLmQikRAJcBNcIOEkQA+HBSgCwgh4b4bajd5ybW6yWlgLCCiETHkJYMWlIdI8iaQLGvmjqnFtrgNO9UzBTodOZkbTCuTfKIGEZ4BpwM+zrvHQuwBks2OL8+ewJw6H7IFCF3Ni3WGoZn2JamR4h5HIJF6wcHHgEo7lMwT68T/E0wovSKVpcLwkVlkraJP8nDXi6bQdXnq6PX3saRK9ovEdDhoHssGjNEpDmkWxKE6HpuSJ7opwXla0RPADqUtrUJxJOnT22IMQSVO9FlKsSAk3Ewfn5NHj3xZB3UxBCNqyF5ZS6gUEWQPl2CJtxAvuo9hfMXRYDpPLx/tRU1mYoE0gBKHepM934fy7PY5KPJYTJifdRZJCCSkPO2KnP6v6CF1HBCcaItAibeDwvOvvihpT6UyoRhVCNB4i92WSBO2rjx+3g4eOtGf/9Fm2Au3ubLfVdbQEyfFDEoV14eku2RHiiCoxInADrquKuatXCBMJbHQPd6g4IVydiK5kt6zm5YXvtsXDmlVK/8CtuVgH2VRdm3l+1w5U+VPuQRnFsZZsP8JweAsl1gyjkbG+bFAwVGvUuZXNSddJNDQTM0hqZbOTcYlKr3ajH+GGmRaa5BrpRYkwdk1ORkhsArcdUJ44cvlcEgVJFQZUgJ9jQznv2qMaBpOCFTrGP8LxObjQXnjuhba6uiLmgqt/5IJT4OLFp5l9H/BwRssYANE99vCrOvkD3nD9TJtBzWGzpbDQwm+kT0LKqNfkGhA2xbGSI6vWXmUItykETASlrm6wJwWyx+HGFITN2Y2QMHS91h60ivMkPGBffPbvU0gWbqzyn9R0Xjqbig2A5xwg/0gc2GlzrjdqpSaEEuPGS8y196dgByugVGPgSLGjSSRQLbtmjVLn8eMnCDaEqn3n5//UfvjS8/LaCb5YEG2XB7+HmUGU13a+vE9Y8NFtOcq+FE6nP4n/DkOzt5hajuXLAtLs3RwqCPW0rFOyma3dq2k6QqpVu7ukE81mMJo1BIkPWKNSviH7ldw6NWlICwsMmg5aJDXNbPhw3H1me6aN9ihtMREAOQAmijfAQGHUKEAkNSoEptCQ+BPCFQdCp1d4ctko3XMmGgj0Ju01ZleEnf/nd95pZ86cbv/4Dz9rf/93f9sWD8+3xUOLnB8GbxueNuNSsCog/jVlCEMbb3TQKR0IWPq7uA1u8Y0GDL02n7Hi0p0jTZMFO1fpvLoNyZzobAVWQbiXJ5N3p6oHHYjbh2nWDJcCQzPeGeu4uLRkLZsSrBy43vi/73RPLl14b1pZimJ/ZZMVf2MjOLBlH8mNPlP6hVPJ8bG+u3G3PfX0U7LplHrFhUlyKMQTLzgkP6paDs8YDRmTEuHA1VSSVC/1Y87sRBPhw3ZwihLnNz7JiIkftKUlTNgB7xlCL/V7YeKuSAKM9nSbrwo26ekOl5uydez88OmjlvJ7xjbG58m/eZ0219bW1zgkhtqFhRiphK6u4/OUHEc1p3aKmJRK0Yoh3aNHjCggvNG0iumFQuUhKpypk0sX3p9ubm4yoTCcrlrBksUeIL0JHSV41wn6ZcNjmwPzGaBD2ShVYSCRrF512g6hNdNWo8+FL3WEY0m8xF/garFeiGQDxiIjiy3BTCZqfjIhXgsoEKxv4lRQXfPkmesFz/fNN1vMpYcbpfssLKjITmcqQA6CwBpKM6eDJQjcVEa6s1vmqGSjKRRutpDGEeZOTJFpNRoeU54pthtTgZL8GTBuJ19szyM0vBc2OxL57U6ZbiZ77hFNpeEbkqVwJCeieucSfgLj+u8rohWFpuJu5ZI9ycBCoSyXwQ8u0EcYR5Sga89hlBHnj+gLagxOk3LvimnxBRN3//5WO3xoUaB7xPHz8+3QPOLgbaVQd7XoOAAYldSnHIw17/6M1kOFHsKDwEQcjHotItG+ptgj4j/AhHDqMMeD/kkn1TPmb6YWoG5PxuNYN8dPoAUPlmCsDZ5JPDShCoFJo4N2+ZPf9s3GpmdTojKrg5bNrp57PNrYOth2Zc6GdqAtBidocN8Zv5S5GS44xGEj1bJDF9zTfaSdB1Q+geJ7OVomk7U9xKhGxZdqm03SvWYI8bzppWIee6IRj/MW3m67HSaBxTDpzhyO8RwqicYBlUPmvHRYD0ImaEh2h3V11gph/ygwKI6Y3A4nPp8VocCgueRmylPrzA7adIV9cFjjNPJk/8fl302JPCzzr5SEGHTGRajlWboPORs9q/5lnxlzLqonKaceJy1pPZ40Oyg1BOLfozatQUgQU8hsc7+Mn8pmRwPd37rfjhw9qkEpHuGgbNkA62Xj6Yi6GY+x+67CIWwe1b5LuECSJgYGGPLOnY127Nix/2f6IgjQz2n4i9qWdhnVO4aedvwQdiE7FzPFOFzODu8xYGI2qRMBMzmG8cA8w9T8Lip5iXhkFg4wvp98eumDGXxCbHNOeAXwRwhy2hmse2J8atjZCHnYvU6mGZmeZ8Eih73zOEP99+yJ8h7FAcLCQ+UlYpAfIMHqwuZ5liNe1/35Lv4c1X3meblJT8+g08HMFNbYyBPlx3MPwZ8hCIFSJSunRFBoJvX5/VqxC2k89jIlKbZ1HAZBmxSDay112jXgHZ+7t7nJwg5VPFuD9sQV68YFnHx8v5c6ocbjIWsBRzEdL5qXIpDPbSfDSYqNnG2pqfYDf8c1qhbQQBi03oxMnDzYQTyjQHH4CBRyjDGiFtImI5SS1BvAaK4xLBJ6v2BSxvuMal7i+TwTFjNdILDdMDlhJkz7boQ6WMpJKI8AAAdhSURBVHeFTPM9/Rqn7SGm2TLZokWOZ87nJ3wJFTxtWl2TCMY4SHD8nO9wf7g6QhVbU70/gokKBbj8VZk1NxaWfAk1xOXLv5/SPhtaEw6x2G+l8gZTQiQvdrtWYvAgyYpF3UeAcpry0hEYwXoH9kzJj9mxilGfta0X8SbOrainFL5xRkhaVL0IQbf0Re8/l6DqkMlOjAVPn5g1aY+5NQmIGss4M5qJEPO5g0MaT8UTrB9ULNYFEUzleckzVXufE571iTnVeqpfLHYYzI442VwXLazv6VYuv2tMwOSzzz7iZsvDEyYq3mtuPLJiY6pMNjvqvnrrWqJxklIQiGpXCJbWnrGxuSayXimPytFTokYxcwowOfXwgBH/Aq9u4rze751JQGFuHAmfoDxiampdOUmdYQORFxdiFT8TJaZBfGFWNudKjbBy7RD+5tBwhBRNgRJSWQtBqPT90cwY7nIsqPP5ps0A4RBKuHpOTQfsozhKQ2OHlGGz8eHqqWbzUz8epzykqFC5QY1kY7Upo+gxWoaG/R/9xFGvtQ5bncR45ji5meKjk5ci/igYxPGSWgRXqVOdTswM4cvfIoiBGAffpsORcIr3Mxl+/02364hFQdGLBFuqM4DGrBlMFd5V5rACE3WvmkmMd5/3UM1cdfZ68GifbVblAMuRC0NEogL+jgs+9Ds+//xc51SpH0p5MKiObE6kKDndqp5rPbyq8bHE+lskOLadoUahg8qmj2sPxCfGIIhZUClQePxaCBPjwvbbYQmNNq6TGrJSkE7d+lQmWRLnbzhW0tUiBxi5+pz4qn6x2XHWlMMPBNgJmd4TDm4ZIV5qwTo2/969LQpGZ2xy/h73TBkzZgIags7XnCpd1T/oG02NZ8QrNjtSk1NWN50pOvdJMzXKAWUhtk0hAY1pGBAumqmqKbJww2kbZdMqEJHq2PiYAZkQJVeGV6xTgRQu0SX2/BGC4GVUsx5hTH+GjGvEe6BZgfPHFCb2cMvJnzwP/qQ69vgFePO5djZoqOtBWJDTCUEJiie16W9zziJAua+c2j2GeEAE6T2Vas7BgBMatNDsgTKYz45sYvfJF1+cFw9anddRSlYjoaHm+AhGbJaVeMc/V6ejhh9V6rT4aQ0a6jhCNpw6lDrdb+wifjYuzxsBVSZPSQdWoAwqYJxpZ4mkcalU5cSYKuvBw4fUEuRutIOVEI4LzchE+Paoea/GjI8Th2q/TzLUveJkkcQP9RxBzmZn8/P9CBQg1keOLLloFKbkUaHTvjjTZh5Xric88//8XDZbLrw+GDWkgsUgcmNhxMWOvExV9yqciAqK0GSX2YT+UP6bed2OIEHixm1GrhvHo8c1hkerNtZasKnhHTZDi2xwIBGv0DI6BQinDh9eGsCA7n8Hj65wCM+IpEo2O2iQnETew5oDahYLOBoAM21wIGarxqwaLhmxmouoMbjWAKp+ND5mPaJpIgSgBHvyyaOMtSHJ/YAZCxw7zh1WnA0vT433mT2ZBIqw0XoBVprc+hNtkOZb/Vt56H5Dj3msKoZ22JmsEepI3qr5iGceCR8/F2xoVqWbu6yGHkUooRJRi0fOLoBJBR8WPlflWBErPK54huQa8g7yA8yYmNGI1hJxxMhs6CRLTqScqoH/jg+E90h0UgWY4bCLRtV5zufzp1S6+VFNeAAPPbTfSSbxmZFBq55xJEc4LcGH5GVrI0EAQ8fEpzbSmbId1zDcV2bQtVfWwQL5d+gngCiJk7V/w7UnmQ44xk50zeLwUvH0MDNYhEMkiEOodJA0mouHl8hJokze6GGTf+DZIrPGr2cBq9kQkFBCzejezmWEPJue39H1k6cfEYUEwKEVhxBopHUEJEIg1a4GSp1wMSly0KyjBX7fh4BTfQEgdXMh9hICMJMujWRp4VVPjuufF+nqPjXYzgIgz5WntcTY+G74TmP0qTWcqWMt24akdk7GpkvCR9twTnwWJPY/mw2nJeqf82bNTMgcOMuhYBnU6GcszsEF0UzVzc6192ukaBeZORMRWJtFSCMEw2fQy+XfEhTXsn0N2nN7/DtZF/8shy+Ck/tqr9CSrGIINS8STNCsPjwo+vJQhEwAanxspLzrYMJif+Nc4PuCz6rmTKkMrpr5ZJUsuTlWCTOJd6vW1H5xX5QZM1YqKjtOVcITLeAgxgkvSxy54cmbiNbsDTwnlPgQ9nlSoPlX8axy2NCgGF6xkf2iBpvF8/YTHRUPXtCcQDx3nLrYeTbulRFMSHAwDGQXrUqwOKXEoO3stKWjRzsQQSHfWMH8HUxK7D1zFm/A39y9KenyaGlV3Kmlocbria6OQiS7OkuxPbKD8F71QJ1+0r9E25yGP6u8uvFU/24zDYlrdVjiE6g47+S+a+PDdAxgdU5U7CliWXB2Yqgc4LoLwHujros6d6V4dmGB7feO1SNssPOY5Y2vsXnjpPJeU+H3EhYpATL4YhB/R4j7oeImSVvBK4eNX1wQ5psACg+hjQboPlCiJm72nAbYl0oe7TS+7/73fRjI9n85OQ8T7wFtAwAAAABJRU5ErkJggg=="/>
+        <xdr:cNvPr id="14" name="AutoShape 14" descr="data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAHsAAACkCAYAAAC3r1GFAAAgAElEQVR4Xmy9B5Sl2VUe+t0c6t7KVZ3TdPfM9ISePIqDRhqhZAn8DMu8hXnPmGXAawHCZDDmwUMYk0GABcY2wQSBSBaSQBKDNJpRGk3OQTOdu7q6ctXN8X/r+/bet+7o+fbqVene/z//Ofvs8O1v75P6ylfuTwaDATKZHDKZDIbDIdLpNHK5HJIkQSqVQqFQ0Fe++Du+n7/j116vh1KppM91u11kUmn0ul1ks1lUqlV0Ox19bjAcYjgcAAkwTPi9XYfXKxaLun7cm+/n/XuDvq7fbbfR6/X1Pl4jneZYEiCd1ec5Xv7ni9eIMfIavC7vw1fcg99zrNlMBvVaDYP+ABOVCjqdDiYnJ7G+vo7+cICpqSmUy2Vdj/95bSRpNJoN/Y3XHQx6+prLZFGv11CpVHQvpNN6P+eB9+X99Cz+lXPG8fErr93v9/X+mAP+rt1u6/7xe36en4n38JHHfx4MbL1qtZq+JgO7ZjabQbFYQurRRz+TJACyvtgcDC/A/5zAmKj4ykXW4g046fZ3CklMLNcAyVDvyWSymkDekO/JZCgIPc46uFx68H6fP6JSqaLZbCCTztjkcuFgg09RQAYDDJNE10mlbHIyubx+jjHwPrwff8eJiYnm2PL5/GjSY3K5yFxwjovCx89SkPj+drercU9MTIwm2+YgrbEUikXdo9Np6bq9Dt8/0PizuSz6w+FIiDlPMU6TBKDVauna/Bs/z+cZF8zYWHr+VErvp4A1Gg1sbW3pd5VK2TadhDBBqWRj5TU5tkzKNif/a30eeeSzCW9EqaBUhzRmMiaNsWt5gZAwDoSf4QXGX3wgTjDfpwE2GppkLn08kIQ+AbLSHKYN4sFarbYmm/fkq8MBZzJoN1vo8/tsVg+RzmYwMzOja8YYOAl8qPHdHRPJa8Ru5vslKJkMEkp9xrQDBW44sPFo0pEaCXOz0USn28G+ffuktXRPLnCvp89QSMoTpp14T16f8xC7lb/jz3x/aAj+HEKgsQ+GWshWp439+/ePtGyMnfcZ9Hsab284sE3A3ZskyOZMI+dzuxsxFlnP0uuaUHGxbQdkkMvGg6eQplhwx2ezI9XDwYeKp3qhpPPv8Qq1rxtQLfUHSHH3+04P6YWEwXYIP8Ndwr/x//b2ttTOxEQF2byZEk5Es9mUFOt+aVPNMRG8X71eH/0cE8txUfXHK8yGFjpJkKdK5GK128hkM0hzTLwfhaBQ1L34GalvQIuhuTIjos/SJHXaHZTKBY2fgspdSIEYN4tUrRT8MIn8Wwidmb8U2u0OUukU8oXCyByFidI4+n3kc3kMYLs1TClNCe/ZbpugmrkbjjZNMZ8zIX7mmYcT7hqqU74K+bzZwIxJTbw4UP6ev6OEUgVJsoecexOOUCGyYbk8qKz5no3NdQ2CExFmQjug29X1ymWqnwES3xm0vnpwV/cxCqp1jqPX7vBxkc3nJQSctGq1OhrruI2L3c3J54Rwgig81CBSdy5wOZoPJBgkplI5YVxYCdtwiKYvYJg3PsfOzo7uqUV0/6DdbWsecrmChIjCzvmlLdd8pmyhzBylpJK5cfjM3ADtTlv+QzzDxsbGSHiq5Qn9jf7EuGngfIdW4XxwLkJ1x9+kbb/ylQeSMp0E38X8pe1YU9vhjPHBeSHZJ19sk54JORJUg8WiSbfZNu6+oSai26V6tuuFitNuGZrTw50sByudNtua0KY1sb21je2dHZSKRRw6dAirG+taBNpH2ihKeKjDuG44llxYTmjsjBi33i/NQ7tb0PWnJie1O+kzFMsVrK+tI1/IY35+fuRvxFyMa69mo4Ecn6/T0Rj17IlNfKfTs53X72sjcY6pwQqFnNQ+BWVlZUXjp/ks5vJaAy4kf8c55e/54nzKbGbMNNCMhXaKv8VGDBPKcfLznA9qPdnsxx57KOGH292+VEkpbxKdSnEf8UY2aDpwox3mNjkmOLzyojsLcsiovodDPSQH1u31sLW5qZv2B2aLudgUECrJGKQW39XpoD+UWjOv1zx/Si2FiLuF+jSdzqDb77k3PpQnigGwuGcR9Tq95kk5W/Ja+wOZjjTv7d5uJksHic5kHu1WC8ikJQx93y0lqdTE7pGixkvrs7LJYcYonM0mVldXUCwUtfuSlO14037uZfNGqZTsLn0AzpG0B4Bex7QOhY8CxMXms/Kz1CKT1arMDl+r6+t6Xr4nbDMFM3yEiFBC8MOZTj355BcTqhpkslJFGdDB4ETa0vZ6HQ2aaom2iu/lhHJgfJBQY1IX3M30SD2Ei5Aq7DE93xAgqTEP7ai+5Xi5d08JplXs9xP5EXxY7cApk9R+zx2gQR/JMNEC8R5JYiGWpCexHVEsFTHw8IxmI5fNabHtfnwiap8ChoNEO3B9Y10LMj83p5+7rbZMVofOkdtwOUU+rjATw56ZQfkrFNi8LUy300V/0Nd9ad/Hwz9+Nmx4q1GX2s8Vzcni83CMVPGcf96v1WhKC4bDG+8L7ztsdcyjaVWLKjS2Z198IqFNkgT1uihkcpK8YWKhQKgLTjofIn7mLih76KAwhwvsNl5T6HFpSLWkjB6jS608U9nOtNSSpLvXe02IRBulsML/ZuaFXrTZPE6IHoKeJr33rsX0nFhei3aWO4LPxWeKUIy7k2q81W5pJ4a3TO3DBdGOTZuqDDVqiwp0JVR2fwvV0nouhYa01VzU4RCFcmm0q/nMNCvhryhUpUD7HAlTGPakbrm4IQAjjZBOj6KWcDLNL8iNsIoILWOueL/Qlvydnv2p5x4RqFIulc1uwzzbcqkgCTdny8IVOSeuiqhCQqJ4oXBcQm3JexwMMOngQ3jo3FUCWuiM0V9JpxRiUUVxYSOc4PWnJyfNi4Q5TXpQJCjkC/LaeX8+JD1pxrdcKKp4TmIsFEO8drulxZVJoK2mk0YB6nYNtODOd+eQO1iefio9MkXUAAp5ej20uh19nhM5HkoVsjkJlRwlmqGUCW84TvGZiGBoMrtde26Fn7Is5vxyTOHAUaD47KGyuXBzc3OvCWUjnAuVH+qb742/6XpPP/eogkw5LcMBCrk8mrU6si6hqbQF5IWCxb5STZykUsnCKk4Mna9koAGN7ARBAvfeIzzjoLk4dPT4PqpIDmK7XhvFvfzM7MwMWu32KKzLc6L7nDhDybiLqRppTkpFQ6K0A4e07ebwaVe4g8j7Npst/Z0mioJRqVb0lYLNC3KHc2KlGt1eT9BLdmSO9+ecMIwUltDrax6klRJaDQN6KMC8Hk0HJYoCxleYNOogaaFOR5+nNy6zZ2/D/PzsSKOG4JvDa6/xWJ6fD78gMA5uAqGh6YzubethplWLzZ2hsCABOq02qpWKSSehR/q83ClpAwG4GNyx3DGx66QmcqZqAjyhMNTq9dd486PY1uFBugU0B4VSUXZ0HC0at4+h8kIoQ7VucXfT4XEAQ0JZNGiXoZs8dtdMXCyzm4kBNPTUM1TBpgWIehEmrUwY3KmFpOYo5PUzr5dn3I+UaRIHXei48aXQldfu9qShKFjTMzOjiGZkN31M1BS8PwEbLUqhgEa9gYmKhad8hWoObcnn5FgVkfR6Ei5uHL4/5t6wCEMWBU7Rdxmak5h66tnHkoBAOVmUODpOmXQKDC3MVqX1gFT18pZztDe2k/h3gg0UgMCF+X6qND68QhXChfLOzRSYM2UOoL6nL0CwJLHYnrY2Yn/6CozZOdGESTWRdK40Jj68LZjtPBfIlMW2HCvtOHetoNax8E82t0sVaVJvCF0GRPEYslBI+FwMnbhr+ZwUBMW57plzgTkHfF5BpA558rliXqYqVY2NWobCymcNDcdn1Wd890tTMqZniOvQzfT0tASJG5DzEoJuzrAJGsdvttxQtRBwrolpV4tkUi+8/IwjaLsgCgdEEF0OBBfL1Qe9VvNg9QtHwMzrJfTJRaEKlQfoi0nEZ2NzwxElG8y41MbgLTGRlwoM3Jzf2QLaAyREy2lfAallhm2cVH7WJm4gf0A+RD6vhSKerJ3q3jd3KLUBF1DXSlnSRzsjbQ6p7bAKehJYe1ZeK9RqxNpyHtMGJnEX8sXvhTJms2hw0YQZ0GegYAwVj4dQclEnpyYtOeTTyvFwiiLMpRAqWnL7G5uEfku9sTNyOu3vKdn78MCZhyBIQ8xEavyZF59OtIiZFPIZokwNvbndaqBcKGEw6KPoWLW8c0mK2Sg+kOBFd3CUpZmYGDkFFBpqCmZcwqYp5u6YrZH5cODGMjp5CY2841xOmoVj4TWofQK14wSGdqA24WfDWYoIIkIcU30ptDud0b1kagbEx7N6BoEghCzTad2Ln+H9+BniCwZYDLBTq7lQM2IxRDGik1TWsk0Ubl6bfoZ2snvcMZ4AP8zh7KM6NWXJIvoXBT4/zUxfmkJ+1MCwBjqTvP7U9PTImTREzoQtwmD+bmS6uhQUcxilgV4++5KEiCBARmrUEBxmcxT0p2jPbUcRXOC2swU39IuCwt9x0gjtlcplhWHh2PDGdQL8zaYGPlGZ0OcD2aIzxJ/lpPCaA3P0qpOTI7+B15eEc9CDvsKi8GojpjR1Y1omJpYIFe0bNUCn05ZfEF5xqG6ZBU9cUBtQi0i1e+aI9k8qME3YNJGGKJWKSIa2kLy/wKVCVosRjlK/w4wefYMsCDYF3Mz3M2oggra1tY2Oe/Czs7MygxGXB6bPZxF27iqeP0sQ220JFneurunp1LDdYSIVy1PLyWY//1TCC+RyWYM23bGhyrTQimogh/Qw0c7iwwp6c4mykMrsnh6eNtRVeG1nR6B+2DA+CCVND5LQqelJYmWvlRk1eJYf53hGgMWQKnoXiTJNZHlzLmAAGgrhaNv1ecPCeT8JL737HLFuy3QxxuZX/p2LaGAPowWOlwtroVOnZ37G0L3xiCzCpvO5OW+0n51O10wLkbY0Q7WugKq+A1S6n4dk/IZhF6OOgKQjvOQut8RMSiqcY+dzxqbgnEYoK83nDhqvR/vOr1wzCgId5Ugppx596pEk0Cthub2+FpXOkGDPrCUMUkyMM1HiMabCINlXUyN0lCSBvnDcoRQMOkemWgwjpvetzJDwdMavGUkdFzqIArHLLRwkNErEzAAOLgr/zpBJpoC73L3rVqcjIeHc8p7joQntI69BoRHSlBhAxPHH/ahOI1mTTpl2IronGzow7TaO7UcsbOrUEibUVFqklAMy/S7o4kWem8/ATcB5irCJX/lZjpfzwu8j8rFM3FDzzh0aYaG0WJ+hZl/+CZ+DIhs+Q2g5aVHOMX2OrzzxsBabEs3kAzOblvUpyIYw7JG7z90c6kJwqKl0hWeesjTPkHivQYMCMnyyeE3loxXSEK60XTk+6GBtmP9HreK5Y4kZUKvtaLG1kxxk4b1MJXeVaJAQuoaIxRMY4lkrM0kWr3Lx5StwEvs9MK6mA0cVST/DQk8TLu2uMUcp1HVMrrJ2SSJvXlEKIxJh8gyxnGDhmTV+Vo6TmxXZW0LGLoiBuMnhYx6AGEOwcTx219iYMWQmMaITwsaDwUhg+RwCv3zTpB5+/MsiL5hX20POSQv5vDkuXGzFa2RtkHLjoRQnmw+hz7ojQlvHvSc141SkwMM5cE4Y6UWUQEocU5sUsJBCxdF8KAdPtOMUqlhYRc1gnrQtgMXLWak8MyW0nwNPF+6SLwK8oE2kAIQTQ01C28nPa/cS5iyUNEFcAD53eODhcYd9DHAj7DavG3FxhEImtDaO8C3CxDUaNWmY0A5M1hAj4M90TCm4XGgKJ0OucAYDIg0oVQAPYWeaNUfslDhyUItaMfyY1GNPP+pMFYt9mSDnhxrNuhaYzgWlqpwv6uE5iAjutbPH+Gjc7bSLyiyNATDSAo6XCzcfZc2C/ODok1N0LMzi5Nv1OB6OY2enprw3BaxQKJoal49AEoGBJYwciGLxPZxkqr+AGyNRMA7YRMxLdWjYQErXpSaIxYisGxcu8PtwgGKxKbTB6qGm0AJ4WBhUKQoRx8+IhQIsP4SIH59xLEbnNRk2hRMs6Nk1JXludHjDBNIp5Pt4T3EISH4grE2giBh8Pi9TKij3iWceSyg5TGVyMFnu7I57fz2qtJYgSdocTly+UEK5zLQl1bqF/nzI0A6GsBm5kDtcUF/CHWuYeAAInHCCFoa42a6MGNESFvQwzQwo/CAE6ULEh+N/20H8m/JAcro0CQRcGC83GqOxxU4Nr5XPKgH0JBCvx8WlL6A42Yl9kXjg89GX4c+2aJaIiMWmg8YF4hgopAzBNzc3R7loOYtyuIxXJ6zdSYYUNGooJm20OMp7M09uiKRsuzuIyk0QtMmksbOzbSEI4+uJsogYEcJFXB+OM7GD1Jce/aJsNrHtGj88HEjd5tMJup22EvrJYIB8sYRSqYzSxASq1UmUJ6Y8xKKDYyqf6pA340LRVlG1cuI6XebELbnP0IYTJKTO0Z7AfkfeKBGxXneESAkJC9za0TeaAJoMjr3bY5zqSBi/IoASU9nKjrmpUa7aKVAUXu7+yJ5xYiIk5ELyvzYA05m9rjhoy8vLyGWY5m3ImYpEBdOvBw7st3yBzBnnxeJ2vm9udlZ+TrNFUqUJI22tOZ4MpxjimQOby+cUVnEHVzwCoqqTQJaK0mB8z6WLF0zbFkpm5sjedSda8+Kw68hmf/mxLyX8ZaO+g067jmGvIyZIPmcTORx0iOojRQaGXPoicoUiKlML8gRJdqA0kiJEOHUwNFQqGCfaCV1yy7bk/Fy4cAGLiwvYs2ePecEOH9KeinjgryAdctdzh8euNrtkSX9OEAkKVOMUDl6P/zlew9oTQY8kSWSFtqVQKhSxtramu3CMAUhEJDCeOQo1zK9rq1c02advuwOf/Ohf49a73iCHs9M2XDoyf+F/MKdgmT9T54pcHCfgV+IOnLdxti43bbtlISIXmxrXHEFuImozmxyxiJIEa2uGIzBvwfmi3S+VLWFFTaJMpUgWBqumHvzS5xLyoNu1bQx6bXQb22g2ami36yCLI5fLmFpk4l057RQq1UkgW/IwKytUh7TeoiQsh3K5guGgj1azhYcffhhveet9MgecUE4+NYFiWIVK3EGkPNmDmUNkHjOFicTDRsPIhJxsqubAyvk3OljdbkdmCJ6WLOSpRSioxptmOElSgBZ0OJR65cQyAgmTwPtywng92UDPpIWD1WvXsLm5gTe+5W34o9/7EN7zDd+MhESO7Z0RHsAJDQHu9Q13N66bRR1yNDNmvgwhsx1Oc2eQr+EMNJvUKPSsFW45Pp9JG75BU8DfUROb+bHsXIZhpwSKiaqszKbRr90UfvTjf5Vk0n3UNtfQbzfQbTN+LYgmw1evb+nMtHO4h4yrBZ4QB88jTbJDvojiRAXF4gRKpYoGJL5VviDItdHpeVrTmBOBo9PmcMEIhHCSRdFxZC5if+4+Tg7NQLvbcWpSRfE3QyXa2Ga9qc9ZmJdCtcpkRV8U2vg9J4PcdArG1tamcHZOEjNh/EwQB8JciF3rW4mfbTS2UdvewA03344/+59/gG/51n+jzygJJC/egB7aawpKs1l/zZgsvcp8g6U9RcaUo2lzIoFwX4S7lbtaCaLQViOMwVk5bhKEySeGFWTyTEUXTJspbBsI8qVzq4TLX/zZf0u2tlfRqW9idqqCen1Hu6TXG2gnKF/NZEQkDpwJkmT5YMwDTyBfKiNXKCObLSCdLSKTy6BanRKVaXpyGps7dUPcFN7Q4zfHy0APc3I4mIhZd4n+fVQqEyIMcFE2tjZx9uxZLC0tKQ/Mscnm0oZlcyjm8zh27BiOHz+O6ekZdFpG/Y3EA2Nnzjb9kJ3ajpH0U4aARXjEcZjGsR3HCadz1GzsYGdzDdfdeCv++i/+DN/2r79LGiLoxeMevj1P1xiwYv0MtYvDJ1EWjQkPX/TAsoMsEk5faDja+OAO0P5qw4CgEfPvpEQXjXiS92oRYhTOy6P/QPuukPnDf/rBBANOWBubqysoTzhJYWjlJ5Q8euIcSHjc4chIEDI5qZpMtoBMlra7gHxxQna9Wp3GxOQCElJkCcP6i+GdqjGodpBCd2ATzAdReU82JwDlxZdewksvvYS1jTX9vecxcuzWcOzGVfHoHtz5JUYPBczPzOL06dO44/Y7BOoEZYcLFHbbgKTirsOWSrQjDB2DdnV9Yw2HT1yPhz57P97xvm82E0LOuUyMOUfhW9Cho8Mlm8xQivj5iPtmi8fn5e/DmVVenqZnQAEzDrrSlA6bCqyhqePadNoCkoQRgMCNcpNmNpywqSSVo2rSJb/xKz+eFLLMTfeRY/oysbonVmGYnbGgPC5CO0Q3n1IXjpI8cd0ASOdyUunZXBmV6iwW9h7FEAa+iKtFe0ywwGNvARwYKmy5cPkSnnnmGZw5c0YL0uoZm4NaRQ/ioVKABLHYoeqCIBDhEgkVfHCKFBedCRSmGMnEvOmmm6QFIg7ns0Y+X0BFwsXxWjKyaTZWsbp0Ea+756347D9+Cm++712iRtEfMNNjfLjIm9PTjjy9tJrnlhU1EATSHBAM4WLtEhW5Uw1MIQ/Acp00WSJe+m4NoCSfI9RMoqcnnpwzyKRPVI44XGj3+LX//P0JbVKxVECKnGXmdJkA8cUhmCV97xmeqMXiLjCuuZH7hCwxFOoPMTk5jUw6j/LUDKbnDmFyZlG5XQoMUbrI1jIuZCjz4osv4oXnn8dOoy5HLZIe8mYdirUFNI6a0Qu5YUzqRy/BmYwc7DchFBa3GzrHF8fBsIg7l/7I1NQ0bjx1CqdvuUVJlYjh47r83M72GlYvncPb3/3PcP+n78edb7pXBX6tesMWeWglReZMmXOpHcl/TvlSalh+gKlxIYb8zMDoTBEi8omocZjgiKcbkFYfxZBD80+4QfVMJC24phDsyhwFMQg3vYFmpn7xA9+TCIhPBihmWQJEN9/LdrSjzdBzNxIrV/VleIeUfDkkeaRdBXECaZyZCJia24NuUsSpW+6SNy4MmA816GNlZRVffvQrePXVV9Go1XVN2mYLxQzgtwW1laMW4WLzRS1iEmsPPVLd/n6S+cY/GzYw3isChvLmNE/GvEwPWVxYwVS1iltuuQWnTp0aZfc4ofXaOlYvnsPdb/46vPLyqzh2/U2y2TQtlrbkeI3kwBeflTl5YeacI3rVjoFHrK9lF2c9IyxD8XmAJq6OhRYWC2hRZauuwoTF5sTSzj4tUtkULoOxeyq62N3ZKaR+6QPflyhWywJDJh6YRRrS1hhFKQj7uyGRTbAyQp7jNpaG2fRR2pDFe4UK0vkqbr37rQIWRLYf9PHZBx/AU089iWa9MWJNWrxrFZ0Kl9xWxWLbw9kuEanPvW89rDMzYzEJqkilxxZ3Idjd2TZ2qVenKvNnyzkbIsg5IaBx04034fbbb8fO6hWsLl3AqZtvQa5YRaFcVdIj8TqrkTlIGS1bfgSdUa6E72gOWz7JWHgU8KuhjtSNxgW0/IFlBM2AkZJlSBsdM1HFXJOEuFui1lBN2/l0DFmk6MLxyz/3/oQDK5XzSDn91x6YWbCWFps7ke+PhAM/Ssg0dlxUUHCHh0dN9d5Psjh7cQXf9h3fJ/L9o08/g8cefwxXl68YgDJWSx1o2jh8GQscO9cEjjvbfIRQ7UNpZ+On0QSxIsScGtMMAlrGXiEUIUghWJaZM3iSU6a8fS6DifIEKqUK9i/M4NSNN+PW2+8UM1aOnlivu4wUwqaMDOhAEZMWS5Z2WaQI2wzyNZzRqw3j5BAurmWwGN6akFD70L5TG3EjjFBGpmhJn/Y5ZMREDSyOn7Sikys4D4Fs/uSP/9ukpKJwMk4oUgPk6FJ5WQztIyU0EhvipzG0cIaJr7iQLKnYtNVqK8eayeHVy1t45zf+n/jkpz+F8+cuaCe3O1TpVpyuHUYO1oi44EkT7TjPJXsFRnjd8uG1K6nGBhh4sZyx12yhtcjK8VqJsNlHI7jF38eFaFybjAtHwKb58gQI1jA+J4tmfmYex6+5BtccPmDeL3qkfouuJIFNzLHV7vTiwVjgKPYzgQzv2ahFgmY7lsAJuJNzTY89dr9COdaBZ4NGxXsa8ZGOXEC8xrBJI0XYlvyBX//Vn0zajQYmq+Sb9QxtoipKvG56wNJQBu4GBngkotooedJEZ+QtkqFhD6b0Jx2GXBk7/RKefv5ZrG1uIDUw4iCxbNpk2maFcz7rsYBhm2PhQtWG6chI4o0LpyyYCmK4iJT0XY41d7+WX3YuhVTGhGfcnsf3sdvHfYBIJ3Lxc1TtBZL3c0bu4KISfi2X5eFP5LK47fQNmJmwShBqiBFU6hUZdLgshbtrPhgDBz4fwEqMyWrJrALGVLz5TwRvbOGNI9DvGRaiOfDUcrBc+DMxc23WD/3mB5LN7XVMVSYsC6UkeQqH9h/Bvn17MDU1o52aLVWMJeElran00PK+nabiPe5WOhgE8pP+EINCFc+/chYvv/yyUpO0J60mHTDzsBV6yNu23Rn2OB6Uv1eO2RhyI0+aP4loPyq8J2Y8MJanY+KBfAnpc7LguJMW34f61jXdU9+140b0I0TJF/EDZIj/M+WbR67AxFBJDpbsvfyeDMrFKrKpIfbNVnDztddKEzDC6QtYoa9jzQqIVyszSIoVee6OM3Ac0nhjPooVRXhRorho1q4EKdvhUTYdqePYHBIW2vVg5Xz6H/4k6XaZ5aIt6WN1dVWkAuKvlCLaHbryzIpJUl18xIPOpOTFmlonamRgQJLL4eJmGy+9+KKcLg6e3mGzaYjPSK0ZlVrvsV1kYU+kN7ngI+ryWDWE/C7PiZvN4mJzZB5aOcGBJsfE3VKioSliYcMsjNvzEDZG/0aiMEdIi6SEQxHFUkVZQC4UVaS0U8YBGAqiV8jksmkUc1nMVSq45aaTgobTXpJLZyvoybLPo1IdY+2qqsRLltR1watCtEPdQeYGi9DLtoQ5hTJhgp4jXrcwL/UXf/RLSqdQCsx+GrbLeqSwlLcAACAASURBVGVKEFWFpQB366t5MzpYVD9cSEuRplApl5CvLqJXrOCVl7+K7Z1tT/dZxobCwCR/qGsuWDgY8RASHKFK9PAt8xYPZ7nrFLIeUlAABfprt7CyMoMBQ5mITp1HF5LOz47b43FPPDJc4dD1B8zpm2PFCSSOzs8TFqbJylcqUum5gvVqSWjC+kaUVIHgwHqqsFxI8zrsygGeLGXx7ne8HSxl5D1VvizqtFWrBpUrtJIxTswkBMxqxY6SeOcAmh/i0qy/8dmiPs1dFqR+4xd+ILHuOlbiQlBBXQdy5FSToGDeLKmzQqpUOG/0YpHbvc0EXaFBfhKl/dfiqYc/j3q7hW6LjpgJCz9HDjZBei6MFtE5zrHrAgkL7jYHH4BNCIF2WYQXopsx+LTnlKOUIZ7kxQgeesX1YyG/NpwLTRM73cIWCwNDy1CdcxMYPFxEkiNzp4wkYzufQsD38FqCdj3lmvI0roiVFM52C1tXL+H2G6/DO9/5Ts/W2diJZ/Mlb97JFRKUsZKrCKtIkmDVjsHYHoV4XxjLqRv3PIAcRQS/9cs/rG1n5D9ic27nvPoiiuRMzbgO99KfiANbrR0MhxnsP/12/N3f/SUyDnZQOxiNyJiTzDoZB4w/m80Sb83VdYRtob7DBsm++w4Zt62pUH9qCUVfg8O3/HHs4PAFIqQLJ2/cRxjH2GMMDKG0WxyNE1qo3LLVUTHTx8RPJl9Chg4se9Kwhj2VQb1hiR9OGGu4FF4hjXTSQ7NeR7u2iU5tE//ym78JJ48ftbptItxO+DAGi5mRICMGrs4oRxx4gkwwGFUl6iRDiMpkcxuVNJFdUzLlv37wP2ixVZfsZD05JE67FewmgMOACM5vgP02EH4uwczR2/DYc1/F6tIr9neVsUTLJ7NrDCcaDcKmJDdSEMx+M24OdR12VWqIVZNy4v7/VYzane5lWu2MIUtc7FDX4Wz972x0/C7s9bizpmuz84SXB+k6LlhRCWI8vDzSuRISpRfJiSvK8TThNAezXGE+voE+bWmvo2Cwtn4VrfqWHLef+g8/aowez9eP8geROxBl2KBYsW2UhevLUMlNUbxOyNXyF7wW7z1OqwoMI/WhX/mhJBZUgIX3BIv6qmBXWALe0pPuH5tXyf+dFvLH34L7P/a3SIYNDZxMC8F3TMnxMwJDDPK02m4Lk0wN79rmcFSsPHfXWePYYkxRQWnjME63TJbHcKGmww+I3bp7bbNv8dz83jJ4RpDQriSvzZEv+QxU105CMNvpoU62YOYuV0A6V0QhVxSIwQVniljz0++jTnIGG24NE2ytLmN7ZxXpwRA/+1M/6R0d6MgydUmVbpskiBARchl2bhiZxeduucliCQfWKckjs0aNOCTjN4/Ub/3iv08YQrCaIfhhu2GPYa8RAoUDZ5JvO55aodnroDZ5E557+CHUayvyUoOcR+FhJ0LtdudHEVMW0N8xcgFDMKk6955t4i15Eeo7FkEL57zvWLyAH9NZW0Q5bWMtu8a97XD2wqEZQZtj8Kny7EwFEqgcYdVWshTqn0V0NqHuw5C/njMiZrqQQy5rxREZr4ztscojGQgf315dRr2xjnwqg//4Yz/ila1dLSQXJgoNZJfFErW+K9FKLNp1EBs3pMyRNufnGZpsXj2/mgYGUh/8T9+nKk5WPoSBskm3zJDZM8szx1dzZAylYrhEqtLmxLV49itfRLOxpsExqWDCYzsyYL4g9wVRn5+ntgjnKHZbnoUEASOSOapWGUZb4kv23MEVLTpBBu4cx8/HwZH4Pr4K2Bgj/MeCh6NmKt18F4Ieso8Ou45/TuPwWD6XLig0Yx6/n5D4UGLnS5RLJEZah0JmyQrZNDZXCRevo5jJ4Sd++AcdLbPuipayNAdTIIwDMOGoKUHkfsS4mQptFlrMwBbWirtW5dxxsWUPnPX5tZ5qEP/dr3fyn4Hz2o3suNDpY/KGd+Lxzz+AixdeRNY9VO5wMk0M6SJD1CoUgjhnHja9cgM1DB40ocupoJBCZa42Q6qAT0cPOQb6K+4nNjDWqoPPFQscKjoctPHnDOctBM5UqAmVFbfbDhnVTHmZrqIRvx93eIoOWybHDJChXKRZFyc1hiafvdVGIZfG9toyavUNlHJ5/NSP/ahrNIIO1Epm7zkHyi94nbnh6bYfd5MlZsi4uagNhNx5HkB22pHMqC9P/ebPvz/hgKluwhGKna3p9fAodpOBdmzlZIxKJgJanT5Ofv2343P/9ABeefZRZNJUw6wVtvJdAhGhsg0T52TKuzDKMLsVhN11hEwqyEOvcDYi2c8HkkMXjXr4wKL5WLw5WgDPzH2tGh/f9eO7elfr2K6WgIAolJVARdGinM+BJzBYo6XSHysglLOWNgHJ5stC3bhjudDKQPXbqG2to1nbUi79R37g+1+jrYLepDVx51g5ctcsMUYrLdrtLxsmRqGqGEAUxF1QSprhN37ue9VAx+LBcFJMYsxT3m2foR3mHYXDzhK9ajVauO6d34Gnn3gWzz/xJXQ77NhgHuHkpBXDGxZuVRoR+1kmJ6V8dixQ5K3lhHmMKiKe57HNSfOiAW8UQGecjk/kt83W72a75FX/bwraQ+XLprmDE9/H5JFLxvdxh4emkJD3jDOnZxqShWPv0SKl89o8SOeQVTtN443xvflsVqyXTquOublZfO93faelI51PF4Idv4tx8e/jYwuTE8JhPpDVltNB5L2ClxDzl/qVD/w7lexavbEjVGNNVqN6kQ8RN+CFFhYWwBYQxWIeSSaHzuQJnLu8ise/8KAexpy6IeYXZ71wwOyWhVKmqqimVNM84lPvdn+IQgOOje0raYMCD4/sFheedj0ctkhphoqORY5F3Q0jvZPDGGWY4+JzRQgY6jBaXkdnhQA4ct5zRmgZm+8RIVSM7w1o046sSWPSnzVGSqrLxj/b4udff/11+OEf/EFfbGO2hJNq/lHAqJ5p9HZlaTmHDDONYxa1cdS6mltH56h9ogpUc/BLP/OdymczbolYkzsnVGXknMnbYq8RPvSo1ssTCCwZquX24NIO8MTnP4Mrly+OgILyBInwjEENFQpEzXZL3hrTpq2nWBD+xu1sOGJmUkIhW2Jf2ACT/DExY4iZdp+XvgYuEJM5vtPDHkc0EL5DaAIrKjRGy8jR89BHvVy8dZeySwlZKabOuU4K1cQxy6g0R/dXjqAuuPRd73o3/vk3vHdMjTMnb+2/FPJGaOpOqXnf5mkr7aww2Xh9Rllwe27fjHiC8WypX/zpf5swSJeKYTG351S5uATuc85bjpCF8bEe2u1jmlNNzzFVwvnuNB556LO48NWXkMomyInUDiwszo2AFAvx0t5vu6ydHdpDu9ix8NiNoY7DpBAXd1/JAIxUImGx1N5uY55Q5fE1JinEJa7Pn2PXCuN3vH40qeS5ec45FtxqoS29Glg2+WEquqcL7tGCqWAjTrCXaTTwEVU6ncKHPvQhlUiHmRPbhw7pWBp2V0CtBp73NQ3rFC0nMHCiJdzeL2a0+B45aSwf+In/OyFXiv27SbpXB6IRMS9tOLSyLN7wLpIQUYutBu9ZdIcJznXm8ORXHsa5l55Ft99GOrHWUlNTE1LZFDcurrzMPqE9a0jL3msGtJiHHwAHB8hdoqY3rE5UV0Dz3G3X7qpxg3stsRI7OhY6zAavN55wGXfUYnF31WhMqoFIRtm1/IBSvS41I+dJZLY0uh0nGoYdbvdUkkP1ru5L0XigVMQHP/hBoYCGVnr1ihMTuKjGOHGKkYeD+tmTM0ZiMAatSIteVGkIk7FUhcwpu5hC6o9/9/9J1HzVS2eEgdDekBJM58JPGMhmmOVJI3EUiQsshIv9vAg2II2vrnbxwvPP4qlHviSCvvBqVmeW2LzVPPKYVLOPhhoV8+wRYrxyld96OBOLEwLAWnH+jTtZsbtHBru7w9E9j+3Gw6zxRRy/7tdqgLh3CA0xcj4rd4xahgRI4YsgJ4222Om84deElookje1QFjQaF+/EyWvwH37sx91OBxXZulOpfwrDWmbt1FLL1HIIp1KqhRyGHWeiOOql4zjU9M+aBFohgiGRCls/9td/mBTLRWTUSwQCBZKEKTfr2zGi73oFQ3qw60QpNEmxwRtj3DSu1od48atn8ehDD2B1ZWmUiy6W8ihPGJPFvHEvuAtb64sbPkOYknEHSw/oD0xvM4SGYyTGzOvGZHxtDB3OllKKXgfN7yMBIgFyGz+uBew6VuhOSFRC5zy34I0x2aNIIW190MI+mgOaRTIIO2u5ezstIY1f//VfwczU9AhsspbfFs4JKQvbzHvGbg/AhbaakYznrpW/GrP1u2RM3ziujVMPff5+IX9q0KL2y757vGwm3H2Lei0nPY4hy6HxdFo/yeHxVy7jSw/8Iy6++qKpmEwa+VxWhQfRp4XccF5OdUjFDLpt6xca6pkTHs1aaU85iVTz47tw3KabJTPHJUKRWPiv1RKx2/lc4/cct7OKSZ0gEOxPYeXBb1NDH2eQuhYZjzLsnhmFWeY505QbCklG7Xd/93fjDW94nXPw9FcRMGge4h7RrYmXFzVpnA3rfPQe07DUKS64chIpcKo5G8rsGcnRk1kPP/JgQk/R0pykYxqYMALhnWLbb1uXWz6keeNx8k5KD8JS3VyuhOcuruIrX3wQLz39+AgUoNQyfjS8mXnznpAhkeDTAyR9CxnGqzPi4aJOy0AZE7RQw5EsYYO+r0XG4vOhHcIPCDX7tSp+3L6H4IzfS8wVz+Pzmv2ehakhMCEs0cFR3HkdTZHHgYMH8KZ77sGdd95h+RWRRUwTRe6BZkkOn0cQ0UslFt9Ewtil9PLDWbOMJVG0XWbqeMtt81E8qfT5z9+fsBMv7aHVPRmfigNSAl0XIqmcRXQseLOeXqxgZH5a2DbhTZ2pUcCVtW18+nOfw/NPPKLUpXUpsm75LMfhBLJVRKdjvcJZE8XidoUT8jDNQYtJCE95F3TZ7T8mQqEcOscH8plRV4TAv3fBEXOc+IpESahsmYgxtC3MQGiPuHcsfpiC2P1a9HYfe/fuxfu///2iHhsM5Pdy+rAEMG3PZxTh3TGxr7uIEuwU6Y3reV+WRRlgYk2AeS91qnAiYtC2rJWJbRoCQcIlIivorcVSD372kwmzVjqRJ2vdh1l7FQDEoGt4axSuST2pgsT7blLd+SEtjDFT6QKefOUM7v/E36Fe2xoxIwnAWO/SrOq2u11SZ62WizaXLzEyHXCJiYoJjh0+PtFy1EZJGh65YDZzHIXiIkZIFRBo7HK+N8xULGjYXA1ojIgYAjCeJ45dd8cdd+DffNu3e67AKjZpQ6PG21SpF+2JXGmYugmZVW8QhwgnkjtcvD0nDHLhtHO9k4L5GAyTdxeVi22JKzp0Rhahn0EBoGoX+vfpf/ibJM3QqdPWLstn85icncYLzz6FYcIwjJBnFXv37ZHtaNU3MUgySGVYrZlHZgDkK2wIYwxPqphXlrfw9x/9G6wuLwlDZ5E4ww+q6Xqt7g3r2BfNeoMOKInOlFEI70kRIy8ECXG3VktxtZzH6LliNnZ0ksAYOTGw5JjIWAC+N6jIdoSUYf29riF8/G9CbdpGCQ5f/NAEHCfr2n7mJ39KY2ZhgHqjD/qqTbfEhqVbWYynpvYD48rzFa1GuLBEIlUbzoZ9Y3kBnVDk7SrDbBCNMzqxaYg0mUHhs+ikBeMPcvz0j4zFk0Lqr/78D5Lq9Ax63bYkgdX611x7Eg/d/wkcP3EKi/sO4+WXX0Q+m8aBw0fx8tOP4/ipm3DxygomJyZw6dXnkJ+YQc/JJCwiT+XzuLzVwSMPfUYdE4kzVCtV84QdoCB0yvBASJDiCqtdGn+Zat/9XahNBXoKKSJDZHlmkiNjUUMtj9vmXe+eMazVnekeHpoY08N7sPjC8prjsWqo0sgw/b8/87OYqU6pw7HUvldi8Hk4FoavfFajEVGT2PtCg9gzMS9hVCRRmdzzj0NtKDChUaTxmPpVBMDuzz2rvuUpB+xVquY6lofv+r34GYFVH/nw/0hm5mbVe2t6egoXzp3DnXe/Dl/8p0+qo++RU7dgmcXvVy/h+tN34IXnnsDJ625Coz3EwsIcHn3gozhx+s0oqEVFHfv278fTX7of5cM34S8+/GEsXVpCPp9RO6geC/ac6cLJ4aFkQnpiQcc93rGFJl4VvTsNVCHQE0wWS4wYkGKCQVNjDppXcnqXYOamJQyBKbN6xc/90G7lzus6Bz1Sq9EiOrEMHR1F64OSYHJqGj/3sz+npEh446ERgnI1KgOWX8IerB3tYIJNpkms0Q0PYlPNupMuIoyjsLIxACneuXzBKkM8VCQMbfQuo25Rm/R40kGpKN+l06xbXThbpdCGs/PC3MI8dra3MT+/gLOvfhU3n74Vzz/5KNqNbVx7+xsx7PZx5sUnceTkDUpyFEtVzC4eQnlyAk9+7mOYmN2L/Ueu02IfO3YUjz7wcUzuO4LOsICP/t1HUaMq8dZV9DKFJMkeGUU2asis04QdTmbVIl5HNebIjHunEarJ3ku1pcSQMTVoFY2aPDXX3c1ta4d7VYWS+4RMM1YjxYlnSMjvdz16i5F5P3rXFk7mVaX5rne+Gwf37hsldsLBJFeNY1LbixZPTjCba9i4naQQfk803+NX7sDwJaiGubhsTBC+C7/yOjqZIA1t0si9B6N0e3vHyCNk/uq4Spbx9pD664/8fjIzO6u2FWxNwSTG8ZPX4crFC1i7/CoOXH8bFucW8NzjX0B5eg6TlUnUG01cc/I00rkMnvvypzTA46ffpAXau/8AXnziATRrNRw59UbMLsxic2MLTz76EL789BksXb6sXWGevrMynMkSB4lG191oWZl4q0h+jhQqPgiPfeAujxYUVu/sPcZGoIsd8Cq1SJUfdc1OiJQqde+fAIXh60Md+CoMWiR9o/bypTiYcbP4vEAubQ1riO2Hz3H06FHccMONygqye1TUG/EZFNuzOW+vp13ISwVMSgRRi+LnpfCrteMsqgcMhZj1d1w0CZu34OTOpkIzSDnB7MysasXYnSoO4su62Uj99V/+j4TF6LWdOqqTVaxeXcbhoyewvbmGK2efw+yBa3H0+LV48ckvoj8E9u87iq3aNvYdOI7iRBlfffJzaOxs4/ANd6HEHT87iwuvPouNy69i7vAp7D98rR7wxScfwKByAB/72Mdw+fKyqb2BdTgO+0Xpj7CEoQapwnzIyLZx8Ny1Ukm0/Q5YyJN2gbFsmLXVjOI4LZYxHV6T16ZajyTQbjLFD5rLG7NVbBSP7y0c9DCR2kQcNW8G7zn3cNCII3CcLHZg/7SJsp1lwrCM5nHYbSmKoa9jdKs0+sMu7Y4EgYe55Qs2N9T/1g/V6r7Y+ULOGokjjZqKKNVpiTVfbPbXrKPJDlM6Xbfgba0HSP35n/5uwqpEa59cBM+Xmp1flId86ZXnUJpawPEbbsH5l55Rw/mFPYfEpZqc2YuFxUWce/ExbK1cxsTiMezZd1iLvXzxPNYvP4t0YQLX3vI2dSB89bkvoNnq4vMvLeP5xx8fqR9BmNHPVOwV271c5JKfFMDfaZFzu0kaIWV+Qq86D3i2R4APTxQKh8lLYwngMOHCtKrRjiyhEWaBqcoAddQtSr3COXF2hgfbVZl9NB+DZT8sMOQiqZuTzibxhgEOdFBQeF/ZVPfCC/kSDh44iONH9mNl+SoOHTupnnArK1dRmShhdfmiHK3DR67BytUVnXaYKxZVhdlt1sVJLzAbmStg2GubZnNIt1CqamytTgvVShkNP6lPWolz9Vd/9jtJvkxyoDVutzjVmrGtXDwnZujJG2/F8tIFbK0sY2ZxrwSjOr2gU/GuXjqLnaUzQLGKhYPXYnZ2Adubq1h69REMBykcOf1mdUQ899LjaO9sYjs7j4985K9Q11FN5pUyZOFXWtp9+/Yr3hYzxI8nZlTGn6lo1ZMz2l97VaaFFlSnFk7xWlJvcaY2QaOx46oihqeaFN3XF5+2UPdxhzHUvFKq7jCypo0aYZzUEeDLOFizGzNb7xQV5jmGoNjeyZgEnt56772YmpyS8DY2LmNicg7XnLwJly+fxc76KvYcPIyt1VVkEx4ydxUz+49jbn4R68vn0ajtoFouQIfjFLhBymh3Gug0a+i1TdAIdnE+Un/xJ/8lId+Z+LUC+X5f9pDhQH19BcNUGvsOn1B/tPUrl5EpltUMNpUpYe/ePdhYX8ba2efFtZo7eB0W9hzAsN/Buee/qCMo9p28HYcOn8CVSy9j+/IZJOVF/PnH78eFM+fQ7Rnezfvu3bcfh09ci/m5eeRy1sEvuv30O9bnrMQDYZx2LBXrP3Px5HQZqXrk8Qu8oPCy+I5xrjea5zPy89FFOECX8URKNKoNgYmkCSnBStHGkY9RPDiWw+Z4IlY3xGs3JByhdrLhPF/T4F8ybCmQxw7OYX7vIdz9unuwvrKEKxfPYe+hw6htbKDb3NKc7T16E0rVKVw5/zLQazGzquKLfGUGM/OL2NlclZlg10rejzSpEos1//T3fzkR31nF3XYqnzrRF/LoNJuC6fbsPyJbsaZMFoeWRbZYxsL8HkFzK+eeV0gxufcYFvcfE3l96dXHsbO5ganFAzh6/BbU6ptYeuUZtb185lIT93/606jvbKDR6eOHfuKnUW8P0B9aX/B+t62meYwfCXiwebwWiIiR0CnGqhazdhjX09apM7E1j+VxVRFeqcpFaUMrciAwRE1g6VaDaMPTDR5XcMnioNnIkAmNU7WqMWIDsKHNpcPJ8NLOFfXTdrx8KFp18/ddnnnqfcfl7XtmXGeSqZdMTxSmQwcP4Z7X3Yna5oaAm15vRwvOse+95laZ3NrmEmqbV9H1as7yzF6kszwQponWzgpSgz62eYpvZRKTc3uQ+uPf+/kknS2gQM/RWQ18eC5Kp832WAkmpxcUpNNpo//KTZUrTmDf3gMCA66cfQHDfhPpyjwOHL4OxXwJaxdfwtrVcyhOT+PaU2/ULl8+/6zUYbtyBL/727+NlbU1fNcP/LjKaLa260ilzYwQwKF3WSa/LUlEqqCw8RpimGZJY2L/MaYQ+xh2efRCH722N9cbU8uWGrXr2kIbYNwmsqdG+EaJChiWX62Az1pYRIYvgI02QxgnSQaiJWqSw7KMcdXbTYV90aXJEiZ23rbF/vZ9HMhqHRSkPVRTwTH1UC0V8N6vvw95HajXQnNnW4zUvcdulTlbXzmP+tZVdFtNadvS9B6Z1+3NDaBXw9ryZWvik6RQnV1E6g9/62cSNpnLuo1MeUaF8KBaMOoQlylkeUh3r42GmCZZtdCYmJyRyqfdbuysI5cvYe/hU4JXV69exOblV8XeYAjGU9uvnHse9Z1VzB64Dn/2N5/EiVM3Y3pxn45n1IEvLEFVKGPg/wghEzrURSGbt3M1szxkhXGmgShpgjE89LxnXYLZs7TXZN6YkGRXNdGKad37p9dPDRKN9tSvLE+wYjCCcFlxysW26CCl7gahBfg7zoslM6xsmDvbnD5r6MfFEA7gvcKjC4Oa0PF0AF7DY2p+r2ILfc5r5HrWFLA6kcc3vOPt6LcaGPa7SJcncOyaWzBIp7B+5Ry2rlxgcY5M4fzB61EqTmCYdFDbWMba1SWFqRSwyvQCUn/wwf+YkKhAiaItYvsIhhNsXqf2Dil6x1UZeXYopoqU9BdLKFen5KVurS+hV6/JBMzuP475hUX1DVu/8JIWYM+J27G4cABXzjyPVnML5YlpPLvcRXlmDp2etd8S89QXkhk224l+aqA7TMzMyXazl6p77oasWSUoEyqceDaHS3kbCi4YPVnZzYT/DeumqdFB65HedWKAWlzJy/YjLbwgYChTMlCOOrSAOYK77BtpAbD7RFvevPkJ1pGY17TkhrUXCdqQBMd9iPBfDDJmVScPaAW+5Rvfi/SgZ+ZtagYHDl6PHoZYv3IejbUr6LGWPJNBdeGYmgT3ei1sXL2IAR01xuoTFZSn5pD6g1/70YROGNtIkFrERVZK06sp1JvDKx0M+7W0W5LKYnJ6CplcEd1WDTsbqzqFoDp/AAcOHlEP1NXzz7PfFqb2X4vZvfuxvXYVm8vn1PZyYt9NuLTdwOb6ttAuJUl27LhFmgp77Ta5s7DL6sO5s4lghSMU5bWMyyWILhQcL71QCpESFd6ey0piTCtQGFhTpSMn/WgK4eXMoHmKUhAoETcJgZU80RsPx5Dawzh1LHw0UkR49LxnOHcBgYawBFrGnyk00gxjPVzlHWWzeM+9b0C1lLPqmvwk9h44KlOyevkVNLau2rNkM6jOHQZDO4ZrO5uX0anXrCd8Lo+JyWmk/tsvfH/CKgZCRTlWIFKUrNLLzqygM5GyKkURERkzisGWQ5GdFgoTGPSaaNW20Go0QCeBi02MdvX8CwoBJhaO4NCx42g2a1i9+AobV6By4HpcqvWwvr5lZaaqELWJ4iIrJednafG+ERLxIQmSiEbknCum9Pi5qNfm7jOWqhMTiaDpyGg7tkH88yGUk9fnlIywMLA7sG4S2ZQVshMjUNJDXYzICvW0qHvhhoFbXpq7qOskD2kYp2AFeV+dFb6mTCcSKiGMwaAJX4Ff3/2W12P/4qzWZXrxKKbmFiVcq5dfRae2au23CnlMzh9BuWTtvzdWz4JUETmZ6Swq0zNIfeg/fXcigqHjyAmbzbK7AltLyzYzCc4qA3c2VFCQIJPn+ZhF2XpOXmN7045xqlaxsO+ornHlwsvoNtaQKc7iwPEbJCjrV86i3+mjtHgMm/2iuFRXr1wxRMhPD7BeXl0hZOEpR1ZMRx555YUQLSpELz5Uk9eoBGU9eJ4q11RmxOKWnuTCkCnCyfDzNpyDprM0WJbkvdA73ThegpSfFnLUbqQww05D4PUUQXS6fta3lSSHLQ8nLnZ34O2RJo0jKFyVuYDasVFxxOV77nsD9sxO6muDMwAAIABJREFUSkUX5w5g3+IBLeLm1bOobSxZGXRviPk9R1GZmsH21ibQ21I0pANwGx39PvVbP/sd1AFyoDgwNokXu8MdDJaeplM5JDnLVVN9m9NCmnAJ7A+mZCNVx9YWUrk8Fg8eEzy4fPEVNLeuIElP4NgN7kEunUW31UV25iBa2WnVSa0sL2uRGA9zt6lGKTPEsD806JBN5ssT4IlEskHecC8otOwWQc+a0Kd2ijxj8uDN+7bOidYWK5L+dK7YYpMTpaSHs2aiSWyUNxGv5vENwx6dKPY86arUNpoXtPtdMw/eKIj4dajigIEjPx8xdhAX6DyFoxhCbQ1sR2WaEuy3vek2LXapNIGpfddgbnpBuYzNlbMYtLcUmRQmJjE1sx/FiSo67SZWll5B3rVVNlfEgIWHH/rAdyZiOaQtO5RmGwmiUZ6xIQKsGmVWJqZTVmzOXaiOPEWUJspuuwaob22LZTo9u4Dq3CK21y6jvrksFHnx0CmUKhWsXTmPZn0HufIc2qX9SkRs7WwpyU71yyOQAokKtRyn+ubyhosTdaKNJVOTqUL5QGOlM2Ez6UOojIZwqx+uqkn1BjTMGFEzWJ8XClZeuLLial88xqqETOkEqTmfU5iUVnXnyrxpO4SdziCzXJEAEVbujFad3R1HZYjM4Od8e8M6TmQc16gx+CE0//xdb0KF53snKew7dBIL83sl1Mvnn0ONNps59HQWE7P7VRde21lDNunIBxLUW5kStzD1X372OxOzOVb0zZBLaFTBHDX2CleaMLFQQkcTqNk5Y/Gy7IF1sx+q9zYHWChXMLfvIHrNbaxcflU2ZfHIDZiZWcT2+pL6irAJfXfqGvkKXGweDcFqTsbtUaHoLbSlVjmZhFE5JmLcUc9katGQNf7nwgX9iMQJ29nBJPXKEYV5u6fvMU896HfkeCrP7nGwbDeb1PJ0wFJeKBfrzsLDVt83liA7kKJkhjtYTGTQOYquhMYPYzLeqFfRwcJy7pGPtwaC8iGcEcr+qd/yjW9DliatWMb8PvO4eZrP1sqrqG+tWPuNdA5z+46qgrTZ2EK7tqbjP3QC4YB14hWkfutnvt11hpXQBhtEh6MzvFExALnZWaTzVn8sJiSTD7Tn5K3xZKC8nYqrcy1KE5if36sdtXb5FbFVJvccxszcgjr4s3mMSIvlEwpVOmxDUa/LuYlcbuDVlvWx8ETd/dkf1Q84CcZKwkXgJDsi1uq27TQgr57kLlVhuoTaGTHe2sPOv+buMz67cs6eCrW4Oiv8nCRJOX19rzrReR5RgUJBs8pSMkeiEQl3KtOl7CYch89F01i69jI3znc3X4MttqzDAgWHWmeyMoH3vO1OTFan0RoMcejoKVQmJrFT28L60lfR7zYFnKTSZWlT9UEb9pB0G1hauiRNUixPYDhII/WbP/2vTY37ohqldRdW1NmWKo/M0OCpFFUYsnho1geMks42URaCMITIozI5h8rkJJbOP492s4nKwkHMzC5qR+6sLVviYvpa9NgxMWV8rJ4X64fHysmXSiY1iBAn04I6e9MSGNwd3Fl0jnhdlsFGaSwFNc77oAqLuF2qUud/GeOFcTX/RuFmbRuJAqq58lBqBIl6fM2TiMPmmrnY7aYcp/Ba41w3LXQO++yVZJTrqLSMggdreGMLLSrx6IjqtDTD1FQV/8c736S5nZxbxNTsfoVXPDu7sXEJnXZNglyd2oPK7KLYNIxqCKrwpGSmr3fqdZRLk9zZ36Fi/MjcREDPiVD44+CCtX5iC1s/c1pnhDA+ZjuJtJrCMUHP9BxDNoIwk/ML2GKXgc01ZAtF7D10UiqPP7MNZmX/ddjqG57MhHuj6Uc9DW0RR6GKdiorTzpIuEu7hpUTEVP7KLbS9J7oXLxI6PBZomCdpkjtuHg3jdvqrWk+goIbTQLkoHq7jvGwyey9dX7UGVrcJN4dOUgQ/MoIYLz/anjaUZAoCpXrU+5sgwGN2B9IG1uAc17vufs0juxbtM2RLePwsetFaNje2cTm1XPotWqoN9uYXdiPdHZCm6DXb2NjdUmhqDUw4Jrlkfq1n/y/VJ8ttTFWlmq4MGucrMsfU53y1kX5zWHo3QJ1oEqprF1ON39re0tYNosGipOzysisLZ1DtlDC/P6junnS62Fnex2Ti4exmSygM+Ahbzy1hhMPdFpNLabSrCsrQsbUUbHfwvbahtSikKiehU089ti47XZS4Hi1pdGS/MSByIJleaotbbkVHhi4stulwPhscYCLV0+6lpFH7WQ/2d047H3sFEE7etF4YSE0VmCw26dVrFvaZTpq6pC4W8BHLcCzWk7fcho3nziMTqsmBK5QncUij+FImGhpY3PlPHrNGjvJoDqziInKnO7RaO6g19rRQQHUVKRIsX9b6hd+9F8RNbbzPoTC++GnnguWeo/KSTVbpUfMHizehsIPbGOF8GR1Uk1pq1PTlldOpTAzN4+rF8+jN+xg76HrpHImiadfWcLk7CLWM3tF9WFMScePue0aKTU6M2tTCRFmgsjk5RENje0dqXvBlElw2g1vHq9uDApSLLx2ZZza5+UycVipOh6JyMIODFGf6ScI+yLuxskegqrbgrFbuctD3ZN9kuJCC//uW6/vsb7qTGqIaDFioBikGqzVfDaDt977Nhw5ehS5BNjavKjsI9X9/IETmJyeQ2o4lBrfuHpOY6YWzZd4tGNFgkuKdrOxiWG3Y4fJcjMih9Sbbj2U3H76JuxZnEW5wGMgbGcYsmTHOUnL+JlVVNuSfB4xIftt8CV42MpE2equqxXtNDam3X/oEFaXltDpt7D/AFG0JiqTU9hcX0OhmMdw6jp0kBOjIzhZdNSIVtG2Moxpt5totWroNNtqkcm/G1drt8JDp+xSCBMoHAv4MXaptFLWIFYdqRB9x7UQdppwf2AkiqhBD7ttTiNtOyfDW2RFoTyv56Wz0jKEPcWMTsk5ox7ghomW21UeLyV2ib2OHz2Kd73rnTrakX7H8089La0wOTcrz7+2eRk7W5tqaLD/6CkU6FUnJG3WsL58Fjwsjru2VJkBUkZy5GIPBy0Mve1GVwfDVZC65YYDyc52DZ1uH3vnp7BvYdKci2Qg7teeuTmxKKpVghpMORpRwFgtwqasFbPjuJwoeucKHZIheEYlJW91dQULe/ag3e6iPDktQiL9vurCYaxiHgl3sLJUHaUtZZO7jFlbaDUbqO1s6G+M5UmOCOyZE0Shi1NpFaOn2bynjEabJTNZxc/WoZ+JClOlPG6AgsoiCNavjRIgsJpoU+27rUWCjCDVOxiiFGd48z00H96TLCNUz2JrhWR+AnAqm0elmMVEtYiDC3tx/fU36Pip8ClUxpMCnnj0EQlloVpFv9XC1tplgGeDF4ooLxwWKbRR20aztYN2bUtzRH8qW6yiVK7aCcHtJrrtJhKCQATApE2ySH3vv7o3YTqvR8eDXYa9+ZyqCr0/mb7qRAErLdGBLf2hFnl6ahJ79u7RQSqGaLGSgtUQrGe2Qv04TqJa5Yl5fRQqVSFOxL6LE5PoVo+h1UuBNWeKibsdLQ4dL8boGxtrGrg87xbP/zLcOcJEqWOPkYm4EeUSEZD1awXrrM+QjQfAqgyHKFjBCIUsT2ZhgEgDNGEeOAU3OxbZ4E1r0MvPTfL0PyJnLhhWnsPr28HqFMZKtYo98wuyvRN54hCb6LR64gIUJmZxww03jLo+EKmjKfvyF76AieokSpOTWuy15fNqbstoZ/bQtfrabtaxvrGiEJbRMdkz1akF7XpD69qq8GFYxnFIjdP3+vkf+iZtEjZmV6rNCXW0wZwk4b7qprRbtald5z1MlaPyqg4V+fnpPTOzM7j2uuvEqCAIYIOwDj4E7SNVqQashTkkU0f1WcbqFBR+JQOD8XOzuY1+u6OfyaYUB9pP9RXgIgDD2leJBOAn7vCe6YxVTPa7BF94CkBJlaOBgKnvJ59HqVbadfNfmC3Ty7NbnFUlJzy2Vh8G92tYp8Wdye4Kx48dU/NZ1p2RYXLoyDVoNxs498LjSPptEGsvTC6iNDGtkwXjUHoWPfL5udiV6pTCrPWVZdRWz9uclWew9+Bx45HvbIrlQ4iaY2r3eiiXp1Am7yCblT3vd5mOrqtdds6Zralf+YlvVehFhUz4Ubli5oVVAdGjhTJnw20UmV4CKFxN8fd2Gp1liSIG5c6k/TLbbwT9bsfO/5pfXJQ22L9/vzx3kh6Ge06LVkumZiQSqKLIrWq0ttDheZs847vZsF2tQ8GNzMAXcXsKJl+BSRND77Pdh0jypFsVBcwwNOFY5ZiNjk00Z288V82Ja+zU7JgI1rn5ATlk41II+PXUtdfhmmuuwebWGmZn5zAxUcX66jIaNfLF+rjx1rtECrx85ln0W3XNyfz+48gVyzh06JA0DL3xKGp89OGH1fF4Ye9BXL54Dq3NS1aDXZzGgaMnNY9rq8syZdnUAM1GU2dwZrLkBvoZpMOekk6N+rZiciat5KP815//ziSqIuwQUivoppo2NTeCeXczSqPOu+pY7b834ELagQkJP/vLSkkNmaOU8e+0pXSoKCjqMcJMenU/7nnft6Pf2UGjZWgWsd3hsCe8emdjw8kTLQmWtWvmrjWP02yxOZb8T4I+zzmhGTFP2QiJKrLzDglBPxpRguh3iOPmJ+QxqZKy9GppghqqjLfde69ds83zQbMoVytaTFasVqozow5Q3HV0Lq+/5Q70Wh1x6evbV6U5D5+4VZNPPjmdVDsdyMptv/DQQ5jU4Xd7sbWxgtrVc6i1apicP6bUMcda49mpTXaeaongQLw+V54VtVspzWSI7Y2r5tekmYqeMELGf/9F9kET3OMkPe/d4VxsoWVaLMNwhdCovYNpOU2hkhCEuaPO2tpRmJPDybfLqwGxeox6aa4awQzVpyWXTuPU130LtjpsoleX3SNEyd5xW5tb2FhdQTLoOH5uxEIuaqdDLNwiAnnebPQeDVr7xLG9/4rCoYHIlJEGDWhW2pr0q4nyqE6d5ufmm2/GwX3k0PdF0ZXjxRMH+fBeU85Qi1jC6soVHSBPUn5UuzS3N3HkhtO4dPY8Bt06NtcuCTy68dZ7sF3bxpEjR3RSImFTWhCO60uf/zymZuYwNbuIrY1VbC29it6wh5m9J7Bn7wHVfK1dPS+NOzs3g1aTMHMH+cqsauTps2ysr6K5sy56mBrv8Yhp+kh/8ts/4H3QbCFUye8Hh9mC+lGAYyfDKhRLeeMcnbgzVP438F1CjwJivGVlnE1l8pSo97ZMgxPuGPqo9CYzgeqJN2qhGVq0CBgM+qpDI6mOtCjmzDfW1zA7M6NDaKKihF2XVP/k7TEMJCGyV1S8ywklXYgPTRvLF0/lLZQKKGSyuPGGG/Du9/4LhXWdTl0EfkPlGBV0lQ3kiwwcqnU+Kz1fmbp0GitLlzC7Z49OGZC6L2Rx9cJFXHPtdVheXkKqR422g6Tfwb6jp2RCWFBRLtuYTY0n+MKDn8P0zCIq07No19ewdO6ryoQdPH6bPPJOc0sHwHaHwPTstNLK/V4TufIMZmfmNa619avi3ak8macPq8Chi9SHf+dHRottIZf3J1HHwziT2k5mGLEhBe0ZnCreGp0kPyhUjEo/RMXAA5oDU+8Ww6Z1noaYrN7OcgSqDFNo5efQyS+g2W6g120pxqYd7zQaaDV3pKZ6ZL2y1kq4vbVfZm7aTtyzXR4ghQANP6ScEOTMzDTWV1clnG99y73Yu3efaYheG7fd9WbVk3OxL1+8LEHrdpog/6xcrSppEW1G5Cc455sTWd/awMziohaRqrY6VcXls2ex//BhrKxela/BoorlC6+iunAIczPzYHRSqfD4KFPj1C5c7AOHjomHT01QX19Gq0Ou+M2YmZ7FkjgCqyhVyRGfx/bGhnh9E9N7MDU5q8UmgsYTkzkHC3v3iU7FRj+pD3/oRxPtwniZiR21QTYQwc/zEp4ah5fa7uBLB6V6laPgVe+sFDndKGS3YwYtAxSokmBFaQ1ChoYuDZmTTU1iY7OJrfqmKE47m+tsrYB2py6An+8jt9zgyzTyaibIrhAFUW/Z8oKeN5242s46zp05o5OD5YB5XzPrMgS0egNcunwF/+67vwf33PMmdfl/5pmnMTc9qaggSn051kbdNAjPqpYvkIJUJ/GAyWpVOALHUSpTnW5gbnYaV5eXsdNo4Prrr7fvazu4/ba7jSY9wR7ljAKsCPHBBx/EqVM3YG1tXdy+2uaqophD192qg1fPnXkG2QSY2seESB61zW3UN1cxtecgZqbnVQ1y9fIl60RZLBnbKE50+JPf/qEkCgREY/VWjdEPk7syXsJ5/Sxt6/tlQqKe2+y0pNaNFAw/US96aXpvci66drtfUI4Z0SQ/F5rHJUl4vM3ygWtuxeKho3j2madw4eISVq5exZXlS3Lc1Bd1dhYnr70OxWwa1UpJMXJc3zh4ea8qoZcgN13OA3ciNYQa1w/TaPUH+PgnPoFbbrkD//7934/6zjr+/u8/gce+8iVzbPw4BjmTxKjzBfHv6E2fOHlCLBoVEKiYzzooMKTiTQnt8kU0jZWdWyR4qClRWTa7Up2wolB30D73uc/h5MnrsHR5SVU4w14T/e4A+07cjG69jo218/IbZvYfFBeP8DFbWk/M7cXePQews7OB2tam5fRlwzkHnpn72z/8aanxAOwjTKKaVk9MERVYrWidjvRSQsEWNGykcrFjjdnMsTPnbVxpWBtn7zzgxxf1ujxxqCTkSCfg+HX3n7wVB/YfRKu2jVy5irnFPejq8BlDuRhFMDR76cmnlOyQifAyXFtb4/AG6udDdxKenxDkDNLBMAfCive9412oba7ghWeexSuvvjRKDgk1pBZKLEMXzeLJsKEfEXRg3mNyakr2mKElNYyYs/W6wkzGv9RGrVYPr3vDG9SEiLmJhKnWYYJHHn3UBHYwRLtZUyODZquDI8euxfLlC+g2a3JoF/fvw8b6ppVZnz+Lyfm9mJmdx9raFW2GcnXaDnuX752oKDD18T/9Oc96xaLEQRu2IHTVY+G4+GKMyMZ46exoMQ0UiMW1isZd+dC1YrZdnYcNZ77ZeG86ZXOUATp43e2YmZlDu76NVg+45uRJk3T2YvF66VaziacfeUSTZbVc5L7HgY8mbAGt8jMqDBiZJdvsSln2SKIs4u4336MzPK5cvIiVlSVD8lhPXSAtyzo5jkwQixG8S6OlVXkd4tI0N9ZhgYJAweDPtPkkVcq5K07ge97/flxz5JhCKAI/HOcjX3kEO7UaSjyLs93E1GRF9fB0tLrNBiaKOVXDTs/PY3V1HYcPH8aV82dQnl4Qf2Dl6iWU8gVx0phfiDPAei0u9of/s+9sSyJwN5jjZd0LvARaDlks+rhaJy4rmk5sei/U293NVNbet2t0wIqfejvWEE622lmgUTZz9NQd4kqz9HRzcxu33nan6EN9LwgkiEsy4PNPPAHjjscZnS6oLm3xe9M+u2duywt2fjzbhPLnm+5+HTavXMH66gq2ttcFCAlhcx5ZtJuyyfImc+54RuPa2OWMAthjbhxyVeTC1hq9Pk6dvg33ft3XabcGBflXf/VXsb25hTvvuh0zs9PSIoRl2W2KHZwD++dYGT9rnaghU8DUzDQ2NjbF0WPju+iwVC6woH8LqU/+5S9rZ4fKDRUbReheyTc6fZ04ehh9U6XehMa98dHnojmNfm9N9ETrkZ0mxkwN63XVbvt1cLiK3kzLnLjpbhRLRXD38nD1O+96I5JhV8QH+ges/OA1n+VikxDo6dlx8zFuRsxRsVMLOOlW62VsWXK3KLQ33nU31i9dxubGGhrNbSUQQiEpDeu9xSJEDWaqJYeM/x5HJGqR3dkN4CoqRukLTc0v4r63fb2gz26jJkH8h099SpwAopTtVlPPvr29uUtXJmihA+ZSgqzvu+8+1Ld3UCiXlG2k+aht76hogI6q2Dre/Sn16b/6oGlXV8dsnRFVhoq7YWCFuFGOhu2abtsZHCQJDeEcGcgSoIqlEE2VxiEzpt9JXrTT4Omhs5uQdxvy9OO1N98tpIxNbzc2d3DrbXcDSR+dtpEWCMgQwHjpxedEpzWYNHaupSo5vjixwMa/Cxrp++iE3DcTdPr1r8fy+fOqH6cTx6DTHDM7mUDM20gWceGdzCAz5R0gomOSiIuuScRC8ffaGEijmcBb3v4eVXU0t9Z03ccefxy1Rt2Yq85eVX23OkuRjGnnoZHvTu4AfQGdlUrT0TUYuNu2UwtOnDgpp3Bxcd5qyD71l7+h0Mt2HA8xsSZpRKFMPXtxwKhPib1P6tDroQlUkJkSXXCDdWEPz2YzfmqdN3qLUMwOHkvbGWx8qQGvgTH8/ckb7/TzNbjYNdxy613I8HRf2h9fbGLNr778guwcXxEh0GdQBYvzxU2VjqnwMSxAdeCevrrlDW/A0pkzKmC0fqm77bkoKrTB6tbsr3EUTjZ9LFctyFjQoh3hZEJj41AkkCvjbe94L7r1DWytXpEwPPfC83aWp1pVG8AVTXEZbYRGMg1h1SnBqOUCc/HJ3AmyhX5uNc0p/cSf/1qiRQ1P2rsKEQZUJkdlMFbgZ573bvM3O/PKbqgDUehgSQ17LjgcNnfOwlFidkgagR2FoxhdYZA5TKQv8+up03eKSUpEbWNzE7fe8Tqp0XZzZ+R4MYw69+orst100kYayk/dNQKGTdiIheI2llpD75fmsTHfcMeduHzuDJo7NU0QkS2xXvzc6+C0x7OEBov7aq60820xdGBtHGrLa7Cu24PP3jCNe97xbgyaTWxcPa/fsuecAVCR0DGuqti23lvNSpssK2lA0mudYwaaIm26r0HsXJnLB//+vxso6lAmOwT7Jhsttv4uAiJ3+lj7Z1eJRtAzMMVjldFiCK/2npzhrTOjxsEqc+axLwWHfULMKzfu+nU33+HYb1uY8Onb7lSIxpZdro+lwi6cPydIlU6aqVNbHMX10VB+jEQYioQecoSOAfjceNedWDpzFvWdHfMxvADBivt3SUu249wshB13tW6pYkvnkshh2IVrQ/YRVTjIurIEb/7692ix15bPSdjOnLHjLWNnhjDp7G3vrhRahfehWuecGF/d2EVc7DA7ETnIdHzm47+XMDgfSv34PyfmaZF0UhzPf/RmMxa4CfHSronuAj6ZvImdOGelqqPJVAdfO+A1doEWX9CrxMkaqovsZ6f63va6N2Nnh2yMLlbX1rD/4GEcPHgE7caO4mpRfns9XL50CVubm+Kgx3LwOgQ4RlI/5liJTOiHoclPdDVObXP9LTdj+dJlMWnIXo0+M+HHBIEhTvIbuWxxGq6r6NGCeZM+Cz0t2WSwM88USeMt73gPeu021pfOCjc4f+6MLbZ7/+FjKKtHAfFW3LbBDGJVqYo2kB9O5+FmNCaK45hTn/rb31EMUSyzH7j5nYb5+jmY0TpSYZLtCd5InQ7Ey7JSHCMKGL2YixkQbOw07QS/VrAzQ3p1Yg6rJxw2NcnN4vSdr8fm5roQI+5sxuF33/1GtOm5wjQQr7G8dEU7W2fZOu891DMfSrsjcHkXKIVSLqD8W4BJR05cg621DaytXFFPEiFRHFsY9TFnVnVZrloDHYxdZ6cGBbRsjeN3Y347S6SHDO5953vEe1+7fEaLfe7Mq4rVJf5+T/lI1ppAOL11d6TZMc0YZA3RrLxvfKzVa6KRz/7D7wsuDXqNUYqNVmyOWCBj9tCjzkTqG8qdGylOs7k6scZzmrb7DR5VViv8Al8AMUIlheYV6+jBqCbVzn4TVtdW1FNlbXUV3d4Q97zlbei22KbROvJz0VZXVnHl8mVRbCOc0iLpQBpXoe4oUXeF+jaBsNEJ8k2l0Wy38cd/9Ee4++7bsY+JDR8bif969miU4/6KnWoQjFwzcdG3xZJAMbN+JFMQHYnLI4Ove8f7MOh2sXLpqxLKC+fOGiHSVf04UBU5i5G/4AUOfA+F3tg2u5z34BGYtkwj9bl//OPXhF6jvp8uwRZnGjFg1NGXUpqN8yzNSVMxgSNmYZ/ouQZyZuc8ewStE+fNhpla2z1wLVpPJEkGt73uDeKNE3VaW1tDu9XHvfe9HT0S6nqsDrHFXt/YwJWLl1R/TafFMl9GJjTeuFdwqurFgJAwLyNAiAxTb8BnThaBlK44dYahu332tG8cZ2k70M/T8uOVAjnUCX0yJxae2nvjUBrqoQze+Pb3Ydjt4erFl2VzL104PypTskNndzsvhUmKbBvVeFCYAwCIsNds9Wtp0akHPv3HCZvEcbEikRF2wj5odjeAjlGHP8XGpto5SOFkyrCYBiDqFUcbSfKVMTMzoZN6vM5bu+s1xQnWYJZlwjfedieuXFkSAZF9vtge+g1vfosQNMba8fCbW1u4dO78qLOhjd+gzXhZZskmWlThcC69gI4cPOLyjCgsRy0RN36dkn3m8UYyJeLqEOZY9N1FlTfgHrlpDyvCsMZ4pC7TQXvj13Nn97B66ava0ctXlrxvmrFr4npxX9G8YiMyeRKaw9GeCNMsNIOyfqbKE6Q+88n/mZi63T2OgWzQkPgIAeiI6Wxt503HJNruND0tD9CPNLJF9ERJADY6dshaPlscGWrcvGe1+VANOFROdN0Nt+DKlcsiGjJe5K3uuvtNKp9ts10jGZnDIXY2t7C0tKTF3t0NnJTdHSV17tWRHKfxvmynh1Dy93TqZA+9twq/l9fL8NLHGyf0CGuIvqD+jCYg9j9UXYAsdhSym0hWtaQzeP1b3y2zd/XCS3LKrl694nQwW2gzpbsHxIiE4EWAHOO42tZ9RjlFrzVztFBj/cw//BFnWotkDEmLcUOiaHPU6DVtao7F+uqsMmYDxxeetczRRYg2kLHsru0O6lOoNNMXcRC7YlI/gJ1O2613vh6XLp5XcbmOccxkcdfdb7Z+afXaCPAgAHLxwsXRafajSXK0xjQNPK7AAAAgAElEQVSvh0puasxb9zg7doUgVMMR5Pw4SCP8OfBvPytr5MCS+KB22t5wncczSSgClTQCR+z8kXBwsQG84b73Soiunrf4+tKli6MTl0zQrKCB9xcnnKiemxRGH6G2Y6FDsEJj8hoSCP578B8/nNhxjP7gzh6hNx8XEgDiKpHzF2dHMakfGoEDVmd890AD4YrEF+fT4j+2prSzSEjmkzepigqj5cSk5PMl3HT6Nly8eAbNWl0IGXfg9TfdgcpkVa24wtPk37mzFYo4C3bX8x1pcn0TDiHVdnw+nMj4uxweXyA70NVACk+YasxU9zIjDIc8XtdZ2wolY0fSNHT8aAr7tKAdJX2ETeL1971P110+94IW++LF82aHw79RGOzZRvWIsYPkLTHz2ub7Sj2PHEKzmnHagFDSz//TR/ycdPPiVJ3IAckxsA5CmhTufH719GE81CiTNLbIeix3vJi14e6WpvAMWZgIo0BZmYyFDLsxOG32DTedxoWLBDi27RhmAi8Ts7jpphuxvbkyMjU8Punc2bPujVvYGBy0sFcGUY6Lnjkv2oVj7SflTwgxtL9FoY5Br6aZI4YOkmOobd4rMoYyYd7VP7xyhXBuhzWSYYJjN9yJ+YUFLJ99XkJx6dIFT8zsEkkS1xaMDKKq1Ha9JX9Cc4+bFX3v8xtRTurBf/qI5mA8WcBBy5UXROdsEpEIqZbd4Pvp8qPdYS6It0o2BIfgCr/GGV0kPASiEzF2TJCpmzghwHb88eMnFFY98MBnMD8zrf7m7V4a3/QvvxU7G1clkRScdqOJJ554VIsklE/OmSNebqujowHllTnvXZ/EBCBsXxAwKBzWsM6OUQqKFT+vfi2+ix3NlyCrSCKQNkcIzY8wGrOcRO+faioshfmD1+DosWuwfJYdKmpYY6gpLWKJFUszO1FEWDjPzbYiC/V1k7Aa0STmdmS7vcFQYA2pLz34vxJzauyhTUpt0qRu2GBdyQlzZlQ3xPeN8dQIpqhk1h0fE9rd3t4SHnVGcI/WVVnYwlDdcX/aTd6/1ezgwsWLytpkSK0Z9lBvDfHP3vcvtLPpuHCR2IjvySfI8DAVqSOYvSWnhMpNk7xgn6jY/fKmvdWlhWzWuzvUfbBrHdUd/T52EcMqdV3gSSd8U2g+PxMkujSquTZbcuq4rOixDmTKU7iLIea5M1psljqNvH47RNPGz8+Lym3FDPaKGF5++2ixw2FmOXAwSCTsX37of8lmW7Yodl4U5zP+cFBE9un/a+vanuuurvM+siXLsrk4zTMdGAghJc0Y22BjoLSZ5rl56kuf+tfkodP/oy+ZydBppkmAkkkoNrbBKdB2aOMB27JsS7Isy/iiy+l8t73XUdEM2JaOfpe9117Xb31LXYzxtLvTwR4pSR9LgEZeVpvIk5QJtIYnSxJVoAiPCgRAGTpVePBnQizc79H2pJ1+/e32zb11xtpsf3n8qF358ss+WSdIVpLteGFyvWrBs9Gx1QzLEJWYoCejJ1QnF0gDa19LpQHqjKhFJoxQa288TyHYI0pGTcI0abtzi+3Ea6+3m1f+pz14uNlu375pG68hOVhPcdqonJo1wXvt0kGTyQ1zlMRifHEtAgP/+MN3kgrhZuGHkB580V4nVu2D1nSxWD8qy8zI1O53tZh/opU2C0nPO2AFfxbJfKjG/Sc8JkA8prHvc+2Vk2dZDHn0OM342+3alSs97MgIKJ7ylAvLCU6uoJuqMgVQalnjmkZYpU2W5jGO3oyI1GY9RamedAnPKBgBlgQAYrQBrquDMNd2JofaqTNvtLWrVwiWYHrYqNVoGBZhzHmukM5OngfohMUh19f+qCAUT57ZynO/+wWRKnFociFCiJ3qRFYLtyAQwOq8k7LtG8fESlBX4QYt2u6nt5kSywXWwpBxCKrTIAeeOEnQjG1VgmeunX7zr1gQQC8TrgPM981ry4ImdfuVCYBKZgw5hC0WsIGLY3oLLbBKrqlmqZ/NiFW/p+RTAh5SWaP6ugaqmwpsu/7tqlfSpTxYmKh+qJ149S0WQkDTvbGx3hEv40gNkASzcp6AoEepYazVuvMe3XYnawc1HrTJCFdU4406pdfZbbRjYdNAUkpt63Pao0T4kvbMueIGFqpBXYstG2SmJicpFFZgrPAAMOq99FyvvfmXpKcAVQe5UnYet6t/RNVoh/9WGFeRMlrsLB7Xx+YJz8AowA9dVTun7iH37Rx6pgNFjQOmS7gV/BHWA3TiVD8Y3j7u1zeIc7vAMgVth3U92E6++jaZHzfvrfNkax9k4uJYZk1xVX6vqGrlPGBf5LDFXPR7JtV7/sN/0TmK+q07ZueAC+1eLv1dthsnAMNJ1K9tUJ5TlXJsaj6nPJ3Zi4C9Vi+YHERsR8hnnLB3rK/TFOfxe6Cu/s53ScRD4va97bb89dV27x7w5KMql7q2RiaBv7Q8g/8aAVdoOODFiU6kqFyT90LSJynwJPoeJUfOjeiD2uwxO2Wp0Y3yReDRo8x55s2ftDsr19rdzVX2d3HsYuaTs4xc0rV9/Sv2L1UwPKfEQLG6BtoEmzf5+KNfWhvY1ibD5FOZE231L3XI/8+Rfjqgh8R0OhlyukAGD3uM6TScqxVbvSdmhJKnV8HERQeGPSyJJvGhaBfCxbz1wlI7eeo1MiHTmWq7beXqdQLzMk1eWkm7O4odKXJhBomotjnAVKatV+jkUIVpSAyPFMbAjqzNkkJNbE2CeY+TyGQAMjoZuqy5W/DEVeAgwufAQjvz5l+3zdvLbXVtpd0Bu7OdUzw7ng8jq6kNSvGoh4LVfyrIWWpVb3YO8uTiuV8RSox4MN7zrPxLavIL6c5E7hoLMsKA2d9KzMffcy4XQkfaSrSpGqCYe8bOzXrII3VL5KYF6e79x+3tH/+EuC1K8nSPNB5Qgdg2fTYmQCpdXrQ96V6lEkVHHDloCWgBYMz43LGHnPGl9ClOTNS3snWKh5FnZ77dzh7Sy2Ql3tPAG8wCwbVFSARPQA4UNvPlk2fb1vptjuVYX7vFe0k51CaMsgeZQNBDMK19F+p9Cgx97TzhF8//2o19Q8fFfZcS1qnqm20Ok3SI7BcQCcDYJHrDO2itfaiGOzaGuz2ocJbgaSAAsy+pxj1+z2kSXH9j61F78y9+3DZuL8s32ttt6+vrbR1jLayZ9LzJHThvwFh40Fv2iCK8KHZ8sAEsBvnm2EBQhuTa+X719mkryc6gUcbpfcv6wCuI40n8gEGIWOOXT73RtlZvtdXby+3uxpr6203Bid8H71miADwLINQcBxFHLQ0Y2WQntKANuHbOo0w+Pvcr48a1oYq2ZSP6ifZb4nvzC0JW5gTq1CTcGDavxsg4DVBlcsaCWvUm2rusmiD935BUeLOS2O5Cte2duXbi1TNtA6dgD1TVjQD61bVbXaYZYbg2YQnqJ7UKKN5JVJcgBhCsadaxlKgpdBTIQYKZcq4SStKOEh/6AbbjIBzQ9TAZQAT5aYHSlaft+6+cbvfvrLW1G1fbPYApe11cCS4Wh+y0Yj16+jNxvN86BzJ/ZjGgzum/fPrJ+/TGe87XKiRqNb8QFYV226ouqtrdpz1mBCI2T+p1oCFHBDAECCafaUerUiRzmFjh3E7QcB1qr5w63TbXV0lnhc1GVeyOwxY9B3qzTBvhWLg/X46odsZwXyWElFoc5EGs1ZcCDXVdSrbOlxPznjCOZV4lQsgOYZydfADhzxi5USUJRPjD195o32zcabevf9XubK5zs3ELMkfVAbR+NojIE08cJeKOJU+/x7etP01BiAAvXvgNN5ujkKIyi0cH0Bq+hG5UjRpf8H2wAbFR+3PN/Ey3s2Mel2J6PVbCL17fTkw2qsezOiszNeLJ3lw7ceYNOmRomwEVFurda+urM2FXMnYUqHjLAe7vW5nkxvPtekq0L9Ze7DEDoTxoLsBtLt61aB8mobxW1G5GfDLxEu44ok1R25cX/4MfneD1bl77st0hnQgcOCFMD3pONvYmpLYH5kWwHy2SZ0a/WOJ/ijsPixIstNkXzv96mrSe0p0eG8GN1WXYQOAZzIEWIc/dL+i71RM/CgujlDjgsb6uM3bJPwe5mQpVct2Kaw2AJHFKa6+cPkuqRoyMPAjH78GDtrJyvTtMqqPbZsXw+zlzOpMAyp8Jl7KIPZal0+I0qHMC1BzklgFJkNPNwIQDaMdcuzppoImY2vSJls4ZAEccoOdefJk+wvWv/ov1akQ2nLyEWjbsL4afu0NEiS3BrWhanOaWMI5iiEJJ5eO7N/7Jxfd6R8jMD913NfqmZgvwcLoYI6ePiDnzCnbDyRWqcn96tGqB5Md1kmvHpU5zCHPTXMeOyvmF9uLLJ4hU2drc4MlGFm7l5o2OF0tdW0I3SADY2xVOb6NjcjK6SQkg0smLaAVqtzQxWoDU8eFChVU5N3TG+ZTDJg2pJoqOI2tz7cixYxza9tX//ne7ufw1JxbSbNmHSpIIDpmG2TSSDsATUIg6Uqj0j+LQGrZMDBCe8dNL70+hluSAqBdbR9Y+kRMgWNioA0gKOwVdyYEdQsNfWlajgns4ZUjTQFoWtegFzKbIRimRoahN4Q2+xEwoTTO/+FT7/kvfaxvra+yUQBsQ+LWHRrFtdMIoaVTxgkeQMJoYU4+GY1nbd6qmx6IKqKiig/B64z26AHf1OTQaPoj2KHGrylZn+Pt0Z9ouf/FF+5uf/rTduHalXfz9b9t3jj3J+QfJjDG9y5aoxmgGIEgWeTxsjvjBRDhss7b/Yx9BDt+0Tf5w+QPS1ygLlLgl+12a9N0JghoqnAJwimUze2xpG8GUnoefiUZaeCxtYkIi60Z6uqlj25O1vOm6Dv8ywdaFvftb2+21s2fb2q3raqnZ2WnLN67xwYW8CdiwJhZ1/yAyldQaoEQKMdWkCzelb6tv/AgKVE0y5EfCaEfSCy7BVP9XNXFxqOqTra7ebh988G/t5PGX2xLYEiDkOLEGIdAEGlARcGgQrorHkdUDH5oig9Tgtd6mOMPJ5oPkQlalLKCzJQeDxlE8iJ2NLRinI7ZbiyeV5nRy/xMbqhYVLXYqO/SwS3IAzxLkClUZF1D57uScITo725N2/NSr7fbNa4T34HpQ4xAOaJioZIQq1AxpKS7v5yBToQz5VTCkVJuTtJqyqCqQpA5dHUuxUth/KSldLHFKwqoejnC2JksYpcB32d0207JnDXAtlQxi+AZ1jfEW2zucQwZoFt6LnSPBCYDwxxXL6lDOL5joCKFXjZmT1sTi4SEB36WtsXTizxj8bEZ+P6FSTz06hNCNh6qUDRd0SDEkXtQUlS6Q8HeceZMwZdYXBEA/Ovn6W+3m8lVgSLlRt26taHE8CObbMoI5BTFVaEmqz68WWzk2KnP63YkBB4/aYqfPBOYMX0ySlNJjDVsxIE8lysIeGJw8b6TcNZJO0n6D37xGBLTNHALPxXArspklQDO2s0NOuHtb95iKZqOCexnhXzFE+8OnH/Bk9w2HNDlbJVumJvpsthIk+jyrRQnF0ozmPHPQL0mpjkoQZosM1TnrIOhfeDC8PPovgi6hSvToIjiNsIEnz7xF/jEAnHEfqPEsdGL5qPP4EdFYET5ojapOa7go10WFGt6fm6PWpkQuNDJOzECFIudO79ydKGSz8xcFLSFpcQiUANq24zjajqMxs+manKCnjXCR/RkEufb6EYKCkpSQMnKrqYjDeWXZbJbnAhEuD8JeLmdw6oZn07PxgiHLaWHzuGdcRp0GKEBuEoP60BbcwwID6HU9WbugJ9FZwhAE6plqEz+bbz9CL9gaxkI+pucKB024OYdp6QFmbV5NinjAePhpeNMzJKmihnvNDpFGUZSQaESCykDHTfrcLJxId7pogfU93Pewiz5xDHNAcmDI6eJ5nMPZt0BZ02WdsjXSXhJysTS5X85FFDhyqk62Ptpicuniu+JUsXwn5qZnTika5bO8XCQuajwbSu1g+yhbaT0SRKUXVQkUdW0yBjX0iPAbniAFD5wGCRI3jIYKRNdcIWgP+sGfnyAPORiI8LV8Q0R1GuCq6hKEjjPLYJON6aID4znaCZ34bwq7bDcWcjbRkky6kiEJtxiuWhBjfxlaudFR3Z9qicY6UXNgpMbhxe608eCkJ67jzmd5YeL8cfMOmDQXc1p69+hen9pbBQN/R6jKwfCXPv5N3qKoKpXWuHnGnOUEx7mQsyUvOw5RVB3SfLAb8sQ1mTYmS6xC4u5OD1QnZvP1gv4Erhz8pVWNcnQkVOP0QHvm+Re4qWBTwtfNWyukn6A3ySxWAAvyVtP7VHFawZlhpHIydTpxo5iT5E5MQ9VG4CvXe48qm0yiT5WRPemw7KwUtuOBQDEK4LFOAqn4OEVtx9xWf6mPniZ0GcIoAYxGpq2HULDEabWU2LFWpTicmV8KnZhata2m09BbXUZlDJ/FaKI0ApL7k4wOJTwxL3naUxcwjQf5ZJ9u3BEErBpBLCRIQiqGRm2+PfEn323PPvccqSTxhRInrscMAMD729tkG8LG0dPmu3gRDaiP/dVwtREbd3SttRP+LSEbBQ8+OzabuYKR/lVUEpNh6k5DruCvJFNY07Cxw0Go5ARjU+P9x//JhufgAcwoBy5Jd534oZm0T5MLH/0rq1483oVdIBs/c+xl2fqm8WYHNMwktQWcZHCNcpSEpYs5Yo5zkMqW4GhhUapDe5EqOQbtO5QJCyEhSsjWOXTDS2AMIRrjTp89S55OfA+c33BQOILJbI1KWcqRxL2hbSKgSiIp0zcSOXIKs8AAEEbFwjT1EK33sMthGrWV8W69JOq05nAexeeuTXOiaF9KF9eMNoWwc/18GPJs+TlOblXz6XaJj9A10acX3p0KYTEQFUmu0AmxPY8nrGFPQwTojZY4mZOBZtKecnIY6/qUZL7IiKPtnTvMgfCgiiU7rWIB1ZDVssp9ILcDWO9UW13RlN6Nu6tkEEJ2j+zDYPhzxSxISy2iMk4anrrN7s2kN9PrhQWiEBotk/KmzMFgYooDV52umLeo/ZiebDYrab16WMD9xdPucbK/V0NevAM2P/kJYO/w/ELhylzVCCsagDabF+bpHl2JSONFv4v1aFRRdDId4xkpCjyV0psD6Ie/0zFQykhT64o9g4MWPDeegW4ZhrK5vpzSphZ+FDUEPFTv2Cuvnmkr167y5e5uronczYkdqjE3K8ZZVNyMcBJOHGrSek+ke/GFgkpMC+7BU4TnOuAikWktYeOl9r35hjhp2BycOxs/x+3MetnJ1MFBfludKTBP7Et3eKf9MG0XES0DRcRN5vQDHM5RtIr2JC22U8JB4cSBnpz78JeKswtTLz3yvZEZktrTw0hy8AAOLQy3ibSl8Wx42cp88TTCMwTkx4uEFRmqBpkSXR+4NQmF79VhROJbSYQA7rXjp063G1e/5qJt3d8gYgVCxdKsNUV6oiPhym0btEBEKhZdqBipSxHQJ2rgOAr3VGX+p5Aoo3Ajpw68brovpBFrgPdmehmzxgszFKpcMS34LBNYKSfjul1/SqBSWuY77Gl2N67fSXNc3NFUxZiWcXhpsy9+/B6LnWH94xksqqOnMp33jqOGFB4+BqaeWdugGVgKbVBnvt+WOO9aJzfM/iwPTveYhMClU8+G972I4kSHEkNbiJlQEjq0x/bOtJ0+c7bdurHMzQH98vr6Gm12TwyRqQnZJRHEQjUne8dqUkh7Jgca5lknjGKumc6oHDe0KjOGR1vSA00TTn93PO+0HkOYMVtLGyikqPyA0e0Slatr6oTCvMmpVVwvhKlgVPiKiYRgwy/Suks4a7TUEy5WL9xoCEnd7NjQ/FCGXW4lZAWSGbUGT5eDUuz49MDeN8DpTBtwVEzKopmDOUhwR4GCqp+w370+sD2AgIAIEepx8+cW2osv/Vm7uyZ2QHCRX7++zDHInNG5s026aPGaisRWeX45atgcYsvIqCBHM0PQsanyDVwx8nShhGVDaOVgIfqginU+H825+uwBhoP4PLBkAQlkrSEQ2fCUhKN2c/BynWQy8X1om5rBjOfdVbYrez22Z+jFk63TkpvGkajA9rSuYlIffh7JlIqEIKiYEs8RN+8xcWcDVp4Ym4CXxwMDyYm5GrhGkitwsLiAbmLTiXHNuKMolZR55pnnid7cxcjG7Yft9q1bYmBIWLgLFWlqjU5eo9HJQXsQLmQikRAJcBNcIOEkQA+HBSgCwgh4b4bajd5ybW6yWlgLCCiETHkJYMWlIdI8iaQLGvmjqnFtrgNO9UzBTodOZkbTCuTfKIGEZ4BpwM+zrvHQuwBks2OL8+ewJw6H7IFCF3Ni3WGoZn2JamR4h5HIJF6wcHHgEo7lMwT68T/E0wovSKVpcLwkVlkraJP8nDXi6bQdXnq6PX3saRK9ovEdDhoHssGjNEpDmkWxKE6HpuSJ7opwXla0RPADqUtrUJxJOnT22IMQSVO9FlKsSAk3Ewfn5NHj3xZB3UxBCNqyF5ZS6gUEWQPl2CJtxAvuo9hfMXRYDpPLx/tRU1mYoE0gBKHepM934fy7PY5KPJYTJifdRZJCCSkPO2KnP6v6CF1HBCcaItAibeDwvOvvihpT6UyoRhVCNB4i92WSBO2rjx+3g4eOtGf/9Fm2Au3ubLfVdbQEyfFDEoV14eku2RHiiCoxInADrquKuatXCBMJbHQPd6g4IVydiK5kt6zm5YXvtsXDmlVK/8CtuVgH2VRdm3l+1w5U+VPuQRnFsZZsP8JweAsl1gyjkbG+bFAwVGvUuZXNSddJNDQTM0hqZbOTcYlKr3ajH+GGmRaa5BrpRYkwdk1ORkhsArcdUJ44cvlcEgVJFQZUgJ9jQznv2qMaBpOCFTrGP8LxObjQXnjuhba6uiLmgqt/5IJT4OLFp5l9H/BwRssYANE99vCrOvkD3nD9TJtBzWGzpbDQwm+kT0LKqNfkGhA2xbGSI6vWXmUItykETASlrm6wJwWyx+HGFITN2Y2QMHS91h60ivMkPGBffPbvU0gWbqzyn9R0Xjqbig2A5xwg/0gc2GlzrjdqpSaEEuPGS8y196dgByugVGPgSLGjSSRQLbtmjVLn8eMnCDaEqn3n5//UfvjS8/LaCb5YEG2XB7+HmUGU13a+vE9Y8NFtOcq+FE6nP4n/DkOzt5hajuXLAtLs3RwqCPW0rFOyma3dq2k6QqpVu7ukE81mMJo1BIkPWKNSviH7ldw6NWlICwsMmg5aJDXNbPhw3H1me6aN9ihtMREAOQAmijfAQGHUKEAkNSoEptCQ+BPCFQdCp1d4ctko3XMmGgj0Ju01ZleEnf/nd95pZ86cbv/4Dz9rf/93f9sWD8+3xUOLnB8GbxueNuNSsCog/jVlCEMbb3TQKR0IWPq7uA1u8Y0GDL02n7Hi0p0jTZMFO1fpvLoNyZzobAVWQbiXJ5N3p6oHHYjbh2nWDJcCQzPeGeu4uLRkLZsSrBy43vi/73RPLl14b1pZimJ/ZZMVf2MjOLBlH8mNPlP6hVPJ8bG+u3G3PfX0U7LplHrFhUlyKMQTLzgkP6paDs8YDRmTEuHA1VSSVC/1Y87sRBPhw3ZwihLnNz7JiIkftKUlTNgB7xlCL/V7YeKuSAKM9nSbrwo26ekOl5uydez88OmjlvJ7xjbG58m/eZ0219bW1zgkhtqFhRiphK6u4/OUHEc1p3aKmJRK0Yoh3aNHjCggvNG0iumFQuUhKpypk0sX3p9ubm4yoTCcrlrBksUeIL0JHSV41wn6ZcNjmwPzGaBD2ShVYSCRrF512g6hNdNWo8+FL3WEY0m8xF/garFeiGQDxiIjiy3BTCZqfjIhXgsoEKxv4lRQXfPkmesFz/fNN1vMpYcbpfssLKjITmcqQA6CwBpKM6eDJQjcVEa6s1vmqGSjKRRutpDGEeZOTJFpNRoeU54pthtTgZL8GTBuJ19szyM0vBc2OxL57U6ZbiZ77hFNpeEbkqVwJCeieucSfgLj+u8rohWFpuJu5ZI9ycBCoSyXwQ8u0EcYR5Sga89hlBHnj+gLagxOk3LvimnxBRN3//5WO3xoUaB7xPHz8+3QPOLgbaVQd7XoOAAYldSnHIw17/6M1kOFHsKDwEQcjHotItG+ptgj4j/AhHDqMMeD/kkn1TPmb6YWoG5PxuNYN8dPoAUPlmCsDZ5JPDShCoFJo4N2+ZPf9s3GpmdTojKrg5bNrp57PNrYOth2Zc6GdqAtBidocN8Zv5S5GS44xGEj1bJDF9zTfaSdB1Q+geJ7OVomk7U9xKhGxZdqm03SvWYI8bzppWIee6IRj/MW3m67HSaBxTDpzhyO8RwqicYBlUPmvHRYD0ImaEh2h3V11gph/ygwKI6Y3A4nPp8VocCgueRmylPrzA7adIV9cFjjNPJk/8fl302JPCzzr5SEGHTGRajlWboPORs9q/5lnxlzLqonKaceJy1pPZ40Oyg1BOLfozatQUgQU8hsc7+Mn8pmRwPd37rfjhw9qkEpHuGgbNkA62Xj6Yi6GY+x+67CIWwe1b5LuECSJgYGGPLOnY127Nix/2f6IgjQz2n4i9qWdhnVO4aedvwQdiE7FzPFOFzODu8xYGI2qRMBMzmG8cA8w9T8Lip5iXhkFg4wvp98eumDGXxCbHNOeAXwRwhy2hmse2J8atjZCHnYvU6mGZmeZ8Eih73zOEP99+yJ8h7FAcLCQ+UlYpAfIMHqwuZ5liNe1/35Lv4c1X3meblJT8+g08HMFNbYyBPlx3MPwZ8hCIFSJSunRFBoJvX5/VqxC2k89jIlKbZ1HAZBmxSDay112jXgHZ+7t7nJwg5VPFuD9sQV68YFnHx8v5c6ocbjIWsBRzEdL5qXIpDPbSfDSYqNnG2pqfYDf8c1qhbQQBi03oxMnDzYQTyjQHH4CBRyjDGiFtImI5SS1BvAaK4xLBJ6v2BSxvuMal7i+TwTFjNdILDdMDlhJkz7boQ6WMpJKI8AAAdhSURBVHeFTPM9/Rqn7SGm2TLZokWOZ87nJ3wJFTxtWl2TCMY4SHD8nO9wf7g6QhVbU70/gokKBbj8VZk1NxaWfAk1xOXLv5/SPhtaEw6x2G+l8gZTQiQvdrtWYvAgyYpF3UeAcpry0hEYwXoH9kzJj9mxilGfta0X8SbOrainFL5xRkhaVL0IQbf0Re8/l6DqkMlOjAVPn5g1aY+5NQmIGss4M5qJEPO5g0MaT8UTrB9ULNYFEUzleckzVXufE571iTnVeqpfLHYYzI442VwXLazv6VYuv2tMwOSzzz7iZsvDEyYq3mtuPLJiY6pMNjvqvnrrWqJxklIQiGpXCJbWnrGxuSayXimPytFTokYxcwowOfXwgBH/Aq9u4rze751JQGFuHAmfoDxiampdOUmdYQORFxdiFT8TJaZBfGFWNudKjbBy7RD+5tBwhBRNgRJSWQtBqPT90cwY7nIsqPP5ps0A4RBKuHpOTQfsozhKQ2OHlGGz8eHqqWbzUz8epzykqFC5QY1kY7Upo+gxWoaG/R/9xFGvtQ5bncR45ji5meKjk5ci/igYxPGSWgRXqVOdTswM4cvfIoiBGAffpsORcIr3Mxl+/02364hFQdGLBFuqM4DGrBlMFd5V5rACE3WvmkmMd5/3UM1cdfZ68GifbVblAMuRC0NEogL+jgs+9Ds+//xc51SpH0p5MKiObE6kKDndqp5rPbyq8bHE+lskOLadoUahg8qmj2sPxCfGIIhZUClQePxaCBPjwvbbYQmNNq6TGrJSkE7d+lQmWRLnbzhW0tUiBxi5+pz4qn6x2XHWlMMPBNgJmd4TDm4ZIV5qwTo2/969LQpGZ2xy/h73TBkzZgIags7XnCpd1T/oG02NZ8QrNjtSk1NWN50pOvdJMzXKAWUhtk0hAY1pGBAumqmqKbJww2kbZdMqEJHq2PiYAZkQJVeGV6xTgRQu0SX2/BGC4GVUsx5hTH+GjGvEe6BZgfPHFCb2cMvJnzwP/qQ69vgFePO5djZoqOtBWJDTCUEJiie16W9zziJAua+c2j2GeEAE6T2Vas7BgBMatNDsgTKYz45sYvfJF1+cFw9anddRSlYjoaHm+AhGbJaVeMc/V6ejhh9V6rT4aQ0a6jhCNpw6lDrdb+wifjYuzxsBVSZPSQdWoAwqYJxpZ4mkcalU5cSYKuvBw4fUEuRutIOVEI4LzchE+Paoea/GjI8Th2q/TzLUveJkkcQP9RxBzmZn8/P9CBQg1keOLLloFKbkUaHTvjjTZh5Xric88//8XDZbLrw+GDWkgsUgcmNhxMWOvExV9yqciAqK0GSX2YT+UP6bed2OIEHixm1GrhvHo8c1hkerNtZasKnhHTZDi2xwIBGv0DI6BQinDh9eGsCA7n8Hj65wCM+IpEo2O2iQnETew5oDahYLOBoAM21wIGarxqwaLhmxmouoMbjWAKp+ND5mPaJpIgSgBHvyyaOMtSHJ/YAZCxw7zh1WnA0vT433mT2ZBIqw0XoBVprc+hNtkOZb/Vt56H5Dj3msKoZ22JmsEepI3qr5iGceCR8/F2xoVqWbu6yGHkUooRJRi0fOLoBJBR8WPlflWBErPK54huQa8g7yA8yYmNGI1hJxxMhs6CRLTqScqoH/jg+E90h0UgWY4bCLRtV5zufzp1S6+VFNeAAPPbTfSSbxmZFBq55xJEc4LcGH5GVrI0EAQ8fEpzbSmbId1zDcV2bQtVfWwQL5d+gngCiJk7V/w7UnmQ44xk50zeLwUvH0MDNYhEMkiEOodJA0mouHl8hJokze6GGTf+DZIrPGr2cBq9kQkFBCzejezmWEPJue39H1k6cfEYUEwKEVhxBopHUEJEIg1a4GSp1wMSly0KyjBX7fh4BTfQEgdXMh9hICMJMujWRp4VVPjuufF+nqPjXYzgIgz5WntcTY+G74TmP0qTWcqWMt24akdk7GpkvCR9twTnwWJPY/mw2nJeqf82bNTMgcOMuhYBnU6GcszsEF0UzVzc6192ukaBeZORMRWJtFSCMEw2fQy+XfEhTXsn0N2nN7/DtZF/8shy+Ck/tqr9CSrGIINS8STNCsPjwo+vJQhEwAanxspLzrYMJif+Nc4PuCz6rmTKkMrpr5ZJUsuTlWCTOJd6vW1H5xX5QZM1YqKjtOVcITLeAgxgkvSxy54cmbiNbsDTwnlPgQ9nlSoPlX8axy2NCgGF6xkf2iBpvF8/YTHRUPXtCcQDx3nLrYeTbulRFMSHAwDGQXrUqwOKXEoO3stKWjRzsQQSHfWMH8HUxK7D1zFm/A39y9KenyaGlV3Kmlocbria6OQiS7OkuxPbKD8F71QJ1+0r9E25yGP6u8uvFU/24zDYlrdVjiE6g47+S+a+PDdAxgdU5U7CliWXB2Yqgc4LoLwHujros6d6V4dmGB7feO1SNssPOY5Y2vsXnjpPJeU+H3EhYpATL4YhB/R4j7oeImSVvBK4eNX1wQ5psACg+hjQboPlCiJm72nAbYl0oe7TS+7/73fRjI9n85OQ8T7wFtAwAAAABJRU5ErkJggg==">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -758,7 +809,13 @@
     <xdr:ext cx="304800" cy="304800"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="AutoShape 14" descr="data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAHsAAACkCAYAAAC3r1GFAAAgAElEQVR4Xmy9B5Sl2VUe+t0c6t7KVZ3TdPfM9ISePIqDRhqhZAn8DMu8hXnPmGXAawHCZDDmwUMYk0GABcY2wQSBSBaSQBKDNJpRGk3OQTOdu7q6ctXN8X/r+/bet+7o+fbqVene/z//Ofvs8O1v75P6ylfuTwaDATKZHDKZDIbDIdLpNHK5HJIkQSqVQqFQ0Fe++Du+n7/j116vh1KppM91u11kUmn0ul1ks1lUqlV0Ox19bjAcYjgcAAkwTPi9XYfXKxaLun7cm+/n/XuDvq7fbbfR6/X1Pl4jneZYEiCd1ec5Xv7ni9eIMfIavC7vw1fcg99zrNlMBvVaDYP+ABOVCjqdDiYnJ7G+vo7+cICpqSmUy2Vdj/95bSRpNJoN/Y3XHQx6+prLZFGv11CpVHQvpNN6P+eB9+X99Cz+lXPG8fErr93v9/X+mAP+rt1u6/7xe36en4n38JHHfx4MbL1qtZq+JgO7ZjabQbFYQurRRz+TJACyvtgcDC/A/5zAmKj4ykXW4g046fZ3CklMLNcAyVDvyWSymkDekO/JZCgIPc46uFx68H6fP6JSqaLZbCCTztjkcuFgg09RQAYDDJNE10mlbHIyubx+jjHwPrwff8eJiYnm2PL5/GjSY3K5yFxwjovCx89SkPj+drercU9MTIwm2+YgrbEUikXdo9Np6bq9Dt8/0PizuSz6w+FIiDlPMU6TBKDVauna/Bs/z+cZF8zYWHr+VErvp4A1Gg1sbW3pd5VK2TadhDBBqWRj5TU5tkzKNif/a30eeeSzCW9EqaBUhzRmMiaNsWt5gZAwDoSf4QXGX3wgTjDfpwE2GppkLn08kIQ+AbLSHKYN4sFarbYmm/fkq8MBZzJoN1vo8/tsVg+RzmYwMzOja8YYOAl8qPHdHRPJa8Ru5vslKJkMEkp9xrQDBW44sPFo0pEaCXOz0USn28G+ffuktXRPLnCvp89QSMoTpp14T16f8xC7lb/jz3x/aAj+HEKgsQ+GWshWp439+/ePtGyMnfcZ9Hsab284sE3A3ZskyOZMI+dzuxsxFlnP0uuaUHGxbQdkkMvGg6eQplhwx2ezI9XDwYeKp3qhpPPv8Qq1rxtQLfUHSHH3+04P6YWEwXYIP8Ndwr/x//b2ttTOxEQF2byZEk5Es9mUFOt+aVPNMRG8X71eH/0cE8txUfXHK8yGFjpJkKdK5GK128hkM0hzTLwfhaBQ1L34GalvQIuhuTIjos/SJHXaHZTKBY2fgspdSIEYN4tUrRT8MIn8Wwidmb8U2u0OUukU8oXCyByFidI4+n3kc3kMYLs1TClNCe/ZbpugmrkbjjZNMZ8zIX7mmYcT7hqqU74K+bzZwIxJTbw4UP6ev6OEUgVJsoecexOOUCGyYbk8qKz5no3NdQ2CExFmQjug29X1ymWqnwES3xm0vnpwV/cxCqp1jqPX7vBxkc3nJQSctGq1OhrruI2L3c3J54Rwgig81CBSdy5wOZoPJBgkplI5YVxYCdtwiKYvYJg3PsfOzo7uqUV0/6DdbWsecrmChIjCzvmlLdd8pmyhzBylpJK5cfjM3ADtTlv+QzzDxsbGSHiq5Qn9jf7EuGngfIdW4XxwLkJ1x9+kbb/ylQeSMp0E38X8pe1YU9vhjPHBeSHZJ19sk54JORJUg8WiSbfZNu6+oSai26V6tuuFitNuGZrTw50sByudNtua0KY1sb21je2dHZSKRRw6dAirG+taBNpH2ihKeKjDuG44llxYTmjsjBi33i/NQ7tb0PWnJie1O+kzFMsVrK+tI1/IY35+fuRvxFyMa69mo4Ecn6/T0Rj17IlNfKfTs53X72sjcY6pwQqFnNQ+BWVlZUXjp/ks5vJaAy4kf8c55e/54nzKbGbMNNCMhXaKv8VGDBPKcfLznA9qPdnsxx57KOGH292+VEkpbxKdSnEf8UY2aDpwox3mNjkmOLzyojsLcsiovodDPSQH1u31sLW5qZv2B2aLudgUECrJGKQW39XpoD+UWjOv1zx/Si2FiLuF+jSdzqDb77k3PpQnigGwuGcR9Tq95kk5W/Ja+wOZjjTv7d5uJksHic5kHu1WC8ikJQx93y0lqdTE7pGixkvrs7LJYcYonM0mVldXUCwUtfuSlO14037uZfNGqZTsLn0AzpG0B4Bex7QOhY8CxMXms/Kz1CKT1arMDl+r6+t6Xr4nbDMFM3yEiFBC8MOZTj355BcTqhpkslJFGdDB4ETa0vZ6HQ2aaom2iu/lhHJgfJBQY1IX3M30SD2Ei5Aq7DE93xAgqTEP7ai+5Xi5d08JplXs9xP5EXxY7cApk9R+zx2gQR/JMNEC8R5JYiGWpCexHVEsFTHw8IxmI5fNabHtfnwiap8ChoNEO3B9Y10LMj83p5+7rbZMVofOkdtwOUU+rjATw56ZQfkrFNi8LUy300V/0Nd9ad/Hwz9+Nmx4q1GX2s8Vzcni83CMVPGcf96v1WhKC4bDG+8L7ztsdcyjaVWLKjS2Z198IqFNkgT1uihkcpK8YWKhQKgLTjofIn7mLih76KAwhwvsNl5T6HFpSLWkjB6jS608U9nOtNSSpLvXe02IRBulsML/ZuaFXrTZPE6IHoKeJr33rsX0nFhei3aWO4LPxWeKUIy7k2q81W5pJ4a3TO3DBdGOTZuqDDVqiwp0JVR2fwvV0nouhYa01VzU4RCFcmm0q/nMNCvhryhUpUD7HAlTGPakbrm4IQAjjZBOj6KWcDLNL8iNsIoILWOueL/Qlvydnv2p5x4RqFIulc1uwzzbcqkgCTdny8IVOSeuiqhCQqJ4oXBcQm3JexwMMOngQ3jo3FUCWuiM0V9JpxRiUUVxYSOc4PWnJyfNi4Q5TXpQJCjkC/LaeX8+JD1pxrdcKKp4TmIsFEO8drulxZVJoK2mk0YB6nYNtODOd+eQO1iefio9MkXUAAp5ej20uh19nhM5HkoVsjkJlRwlmqGUCW84TvGZiGBoMrtde26Fn7Is5vxyTOHAUaD47KGyuXBzc3OvCWUjnAuVH+qb742/6XpPP/eogkw5LcMBCrk8mrU6si6hqbQF5IWCxb5STZykUsnCKk4Mna9koAGN7ARBAvfeIzzjoLk4dPT4PqpIDmK7XhvFvfzM7MwMWu32KKzLc6L7nDhDybiLqRppTkpFQ6K0A4e07ebwaVe4g8j7Npst/Z0mioJRqVb0lYLNC3KHc2KlGt1eT9BLdmSO9+ecMIwUltDrax6klRJaDQN6KMC8Hk0HJYoCxleYNOogaaFOR5+nNy6zZ2/D/PzsSKOG4JvDa6/xWJ6fD78gMA5uAqGh6YzubethplWLzZ2hsCABOq02qpWKSSehR/q83ClpAwG4GNyx3DGx66QmcqZqAjyhMNTq9dd486PY1uFBugU0B4VSUXZ0HC0at4+h8kIoQ7VucXfT4XEAQ0JZNGiXoZs8dtdMXCyzm4kBNPTUM1TBpgWIehEmrUwY3KmFpOYo5PUzr5dn3I+UaRIHXei48aXQldfu9qShKFjTMzOjiGZkN31M1BS8PwEbLUqhgEa9gYmKhad8hWoObcnn5FgVkfR6Ei5uHL4/5t6wCEMWBU7Rdxmak5h66tnHkoBAOVmUODpOmXQKDC3MVqX1gFT18pZztDe2k/h3gg0UgMCF+X6qND68QhXChfLOzRSYM2UOoL6nL0CwJLHYnrY2Yn/6CozZOdGESTWRdK40Jj68LZjtPBfIlMW2HCvtOHetoNax8E82t0sVaVJvCF0GRPEYslBI+FwMnbhr+ZwUBMW57plzgTkHfF5BpA558rliXqYqVY2NWobCymcNDcdn1Wd890tTMqZniOvQzfT0tASJG5DzEoJuzrAJGsdvttxQtRBwrolpV4tkUi+8/IwjaLsgCgdEEF0OBBfL1Qe9VvNg9QtHwMzrJfTJRaEKlQfoi0nEZ2NzwxElG8y41MbgLTGRlwoM3Jzf2QLaAyREy2lfAallhm2cVH7WJm4gf0A+RD6vhSKerJ3q3jd3KLUBF1DXSlnSRzsjbQ6p7bAKehJYe1ZeK9RqxNpyHtMGJnEX8sXvhTJms2hw0YQZ0GegYAwVj4dQclEnpyYtOeTTyvFwiiLMpRAqWnL7G5uEfku9sTNyOu3vKdn78MCZhyBIQ8xEavyZF59OtIiZFPIZokwNvbndaqBcKGEw6KPoWLW8c0mK2Sg+kOBFd3CUpZmYGDkFFBpqCmZcwqYp5u6YrZH5cODGMjp5CY2841xOmoVj4TWofQK14wSGdqA24WfDWYoIIkIcU30ptDud0b1kagbEx7N6BoEghCzTad2Ln+H9+BniCwZYDLBTq7lQM2IxRDGik1TWsk0Ubl6bfoZ2snvcMZ4AP8zh7KM6NWXJIvoXBT4/zUxfmkJ+1MCwBjqTvP7U9PTImTREzoQtwmD+bmS6uhQUcxilgV4++5KEiCBARmrUEBxmcxT0p2jPbUcRXOC2swU39IuCwt9x0gjtlcplhWHh2PDGdQL8zaYGPlGZ0OcD2aIzxJ/lpPCaA3P0qpOTI7+B15eEc9CDvsKi8GojpjR1Y1omJpYIFe0bNUCn05ZfEF5xqG6ZBU9cUBtQi0i1e+aI9k8qME3YNJGGKJWKSIa2kLy/wKVCVosRjlK/w4wefYMsCDYF3Mz3M2oggra1tY2Oe/Czs7MygxGXB6bPZxF27iqeP0sQ220JFneurunp1LDdYSIVy1PLyWY//1TCC+RyWYM23bGhyrTQimogh/Qw0c7iwwp6c4mykMrsnh6eNtRVeG1nR6B+2DA+CCVND5LQqelJYmWvlRk1eJYf53hGgMWQKnoXiTJNZHlzLmAAGgrhaNv1ecPCeT8JL737HLFuy3QxxuZX/p2LaGAPowWOlwtroVOnZ37G0L3xiCzCpvO5OW+0n51O10wLkbY0Q7WugKq+A1S6n4dk/IZhF6OOgKQjvOQut8RMSiqcY+dzxqbgnEYoK83nDhqvR/vOr1wzCgId5Ugppx596pEk0Cthub2+FpXOkGDPrCUMUkyMM1HiMabCINlXUyN0lCSBvnDcoRQMOkemWgwjpvetzJDwdMavGUkdFzqIArHLLRwkNErEzAAOLgr/zpBJpoC73L3rVqcjIeHc8p7joQntI69BoRHSlBhAxPHH/ahOI1mTTpl2IronGzow7TaO7UcsbOrUEibUVFqklAMy/S7o4kWem8/ATcB5irCJX/lZjpfzwu8j8rFM3FDzzh0aYaG0WJ+hZl/+CZ+DIhs+Q2g5aVHOMX2OrzzxsBabEs3kAzOblvUpyIYw7JG7z90c6kJwqKl0hWeesjTPkHivQYMCMnyyeE3loxXSEK60XTk+6GBtmP9HreK5Y4kZUKvtaLG1kxxk4b1MJXeVaJAQuoaIxRMY4lkrM0kWr3Lx5StwEvs9MK6mA0cVST/DQk8TLu2uMUcp1HVMrrJ2SSJvXlEKIxJh8gyxnGDhmTV+Vo6TmxXZW0LGLoiBuMnhYx6AGEOwcTx219iYMWQmMaITwsaDwUhg+RwCv3zTpB5+/MsiL5hX20POSQv5vDkuXGzFa2RtkHLjoRQnmw+hz7ojQlvHvSc141SkwMM5cE4Y6UWUQEocU5sUsJBCxdF8KAdPtOMUqlhYRc1gnrQtgMXLWak8MyW0nwNPF+6SLwK8oE2kAIQTQ01C28nPa/cS5iyUNEFcAD53eODhcYd9DHAj7DavG3FxhEImtDaO8C3CxDUaNWmY0A5M1hAj4M90TCm4XGgKJ0OucAYDIg0oVQAPYWeaNUfslDhyUItaMfyY1GNPP+pMFYt9mSDnhxrNuhaYzgWlqpwv6uE5iAjutbPH+Gjc7bSLyiyNATDSAo6XCzcfZc2C/ODok1N0LMzi5Nv1OB6OY2enprw3BaxQKJoal49AEoGBJYwciGLxPZxkqr+AGyNRMA7YRMxLdWjYQErXpSaIxYisGxcu8PtwgGKxKbTB6qGm0AJ4WBhUKQoRx8+IhQIsP4SIH59xLEbnNRk2hRMs6Nk1JXludHjDBNIp5Pt4T3EISH4grE2giBh8Pi9TKij3iWceSyg5TGVyMFnu7I57fz2qtJYgSdocTly+UEK5zLQl1bqF/nzI0A6GsBm5kDtcUF/CHWuYeAAInHCCFoa42a6MGNESFvQwzQwo/CAE6ULEh+N/20H8m/JAcro0CQRcGC83GqOxxU4Nr5XPKgH0JBCvx8WlL6A42Yl9kXjg89GX4c+2aJaIiMWmg8YF4hgopAzBNzc3R7loOYtyuIxXJ6zdSYYUNGooJm20OMp7M09uiKRsuzuIyk0QtMmksbOzbSEI4+uJsogYEcJFXB+OM7GD1Jce/aJsNrHtGj88HEjd5tMJup22EvrJYIB8sYRSqYzSxASq1UmUJ6Y8xKKDYyqf6pA340LRVlG1cuI6XebELbnP0IYTJKTO0Z7AfkfeKBGxXneESAkJC9za0TeaAJoMjr3bY5zqSBi/IoASU9nKjrmpUa7aKVAUXu7+yJ5xYiIk5ELyvzYA05m9rjhoy8vLyGWY5m3ImYpEBdOvBw7st3yBzBnnxeJ2vm9udlZ+TrNFUqUJI22tOZ4MpxjimQOby+cUVnEHVzwCoqqTQJaK0mB8z6WLF0zbFkpm5sjedSda8+Kw68hmf/mxLyX8ZaO+g067jmGvIyZIPmcTORx0iOojRQaGXPoicoUiKlML8gRJdqA0kiJEOHUwNFQqGCfaCV1yy7bk/Fy4cAGLiwvYs2ePecEOH9KeinjgryAdctdzh8euNrtkSX9OEAkKVOMUDl6P/zlew9oTQY8kSWSFtqVQKhSxtramu3CMAUhEJDCeOQo1zK9rq1c02advuwOf/Ohf49a73iCHs9M2XDoyf+F/MKdgmT9T54pcHCfgV+IOnLdxti43bbtlISIXmxrXHEFuImozmxyxiJIEa2uGIzBvwfmi3S+VLWFFTaJMpUgWBqumHvzS5xLyoNu1bQx6bXQb22g2ami36yCLI5fLmFpk4l057RQq1UkgW/IwKytUh7TeoiQsh3K5guGgj1azhYcffhhveet9MgecUE4+NYFiWIVK3EGkPNmDmUNkHjOFicTDRsPIhJxsqubAyvk3OljdbkdmCJ6WLOSpRSioxptmOElSgBZ0OJR65cQyAgmTwPtywng92UDPpIWD1WvXsLm5gTe+5W34o9/7EN7zDd+MhESO7Z0RHsAJDQHu9Q13N66bRR1yNDNmvgwhsx1Oc2eQr+EMNJvUKPSsFW45Pp9JG75BU8DfUROb+bHsXIZhpwSKiaqszKbRr90UfvTjf5Vk0n3UNtfQbzfQbTN+LYgmw1evb+nMtHO4h4yrBZ4QB88jTbJDvojiRAXF4gRKpYoGJL5VviDItdHpeVrTmBOBo9PmcMEIhHCSRdFxZC5if+4+Tg7NQLvbcWpSRfE3QyXa2Ga9qc9ZmJdCtcpkRV8U2vg9J4PcdArG1tamcHZOEjNh/EwQB8JciF3rW4mfbTS2UdvewA03344/+59/gG/51n+jzygJJC/egB7aawpKs1l/zZgsvcp8g6U9RcaUo2lzIoFwX4S7lbtaCaLQViOMwVk5bhKEySeGFWTyTEUXTJspbBsI8qVzq4TLX/zZf0u2tlfRqW9idqqCen1Hu6TXG2gnKF/NZEQkDpwJkmT5YMwDTyBfKiNXKCObLSCdLSKTy6BanRKVaXpyGps7dUPcFN7Q4zfHy0APc3I4mIhZd4n+fVQqEyIMcFE2tjZx9uxZLC0tKQ/Mscnm0oZlcyjm8zh27BiOHz+O6ekZdFpG/Y3EA2Nnzjb9kJ3ajpH0U4aARXjEcZjGsR3HCadz1GzsYGdzDdfdeCv++i/+DN/2r79LGiLoxeMevj1P1xiwYv0MtYvDJ1EWjQkPX/TAsoMsEk5faDja+OAO0P5qw4CgEfPvpEQXjXiS92oRYhTOy6P/QPuukPnDf/rBBANOWBubqysoTzhJYWjlJ5Q8euIcSHjc4chIEDI5qZpMtoBMlra7gHxxQna9Wp3GxOQCElJkCcP6i+GdqjGodpBCd2ATzAdReU82JwDlxZdewksvvYS1jTX9vecxcuzWcOzGVfHoHtz5JUYPBczPzOL06dO44/Y7BOoEZYcLFHbbgKTirsOWSrQjDB2DdnV9Yw2HT1yPhz57P97xvm82E0LOuUyMOUfhW9Cho8Mlm8xQivj5iPtmi8fn5e/DmVVenqZnQAEzDrrSlA6bCqyhqePadNoCkoQRgMCNcpNmNpywqSSVo2rSJb/xKz+eFLLMTfeRY/oysbonVmGYnbGgPC5CO0Q3n1IXjpI8cd0ASOdyUunZXBmV6iwW9h7FEAa+iKtFe0ywwGNvARwYKmy5cPkSnnnmGZw5c0YL0uoZm4NaRQ/ioVKABLHYoeqCIBDhEgkVfHCKFBedCRSmGMnEvOmmm6QFIg7ns0Y+X0BFwsXxWjKyaTZWsbp0Ea+756347D9+Cm++712iRtEfMNNjfLjIm9PTjjy9tJrnlhU1EATSHBAM4WLtEhW5Uw1MIQ/Acp00WSJe+m4NoCSfI9RMoqcnnpwzyKRPVI44XGj3+LX//P0JbVKxVECKnGXmdJkA8cUhmCV97xmeqMXiLjCuuZH7hCwxFOoPMTk5jUw6j/LUDKbnDmFyZlG5XQoMUbrI1jIuZCjz4osv4oXnn8dOoy5HLZIe8mYdirUFNI6a0Qu5YUzqRy/BmYwc7DchFBa3GzrHF8fBsIg7l/7I1NQ0bjx1CqdvuUVJlYjh47r83M72GlYvncPb3/3PcP+n78edb7pXBX6tesMWeWglReZMmXOpHcl/TvlSalh+gKlxIYb8zMDoTBEi8omocZjgiKcbkFYfxZBD80+4QfVMJC24phDsyhwFMQg3vYFmpn7xA9+TCIhPBihmWQJEN9/LdrSjzdBzNxIrV/VleIeUfDkkeaRdBXECaZyZCJia24NuUsSpW+6SNy4MmA816GNlZRVffvQrePXVV9Go1XVN2mYLxQzgtwW1laMW4WLzRS1iEmsPPVLd/n6S+cY/GzYw3isChvLmNE/GvEwPWVxYwVS1iltuuQWnTp0aZfc4ofXaOlYvnsPdb/46vPLyqzh2/U2y2TQtlrbkeI3kwBeflTl5YeacI3rVjoFHrK9lF2c9IyxD8XmAJq6OhRYWC2hRZauuwoTF5sTSzj4tUtkULoOxeyq62N3ZKaR+6QPflyhWywJDJh6YRRrS1hhFKQj7uyGRTbAyQp7jNpaG2fRR2pDFe4UK0vkqbr37rQIWRLYf9PHZBx/AU089iWa9MWJNWrxrFZ0Kl9xWxWLbw9kuEanPvW89rDMzYzEJqkilxxZ3Idjd2TZ2qVenKvNnyzkbIsg5IaBx04034fbbb8fO6hWsLl3AqZtvQa5YRaFcVdIj8TqrkTlIGS1bfgSdUa6E72gOWz7JWHgU8KuhjtSNxgW0/IFlBM2AkZJlSBsdM1HFXJOEuFui1lBN2/l0DFmk6MLxyz/3/oQDK5XzSDn91x6YWbCWFps7ke+PhAM/Ssg0dlxUUHCHh0dN9d5Psjh7cQXf9h3fJ/L9o08/g8cefwxXl68YgDJWSx1o2jh8GQscO9cEjjvbfIRQ7UNpZ+On0QSxIsScGtMMAlrGXiEUIUghWJaZM3iSU6a8fS6DifIEKqUK9i/M4NSNN+PW2+8UM1aOnlivu4wUwqaMDOhAEZMWS5Z2WaQI2wzyNZzRqw3j5BAurmWwGN6akFD70L5TG3EjjFBGpmhJn/Y5ZMREDSyOn7Sikys4D4Fs/uSP/9ukpKJwMk4oUgPk6FJ5WQztIyU0EhvipzG0cIaJr7iQLKnYtNVqK8eayeHVy1t45zf+n/jkpz+F8+cuaCe3O1TpVpyuHUYO1oi44EkT7TjPJXsFRnjd8uG1K6nGBhh4sZyx12yhtcjK8VqJsNlHI7jF38eFaFybjAtHwKb58gQI1jA+J4tmfmYex6+5BtccPmDeL3qkfouuJIFNzLHV7vTiwVjgKPYzgQzv2ahFgmY7lsAJuJNzTY89dr9COdaBZ4NGxXsa8ZGOXEC8xrBJI0XYlvyBX//Vn0zajQYmq+Sb9QxtoipKvG56wNJQBu4GBngkotooedJEZ+QtkqFhD6b0Jx2GXBk7/RKefv5ZrG1uIDUw4iCxbNpk2maFcz7rsYBhm2PhQtWG6chI4o0LpyyYCmK4iJT0XY41d7+WX3YuhVTGhGfcnsf3sdvHfYBIJ3Lxc1TtBZL3c0bu4KISfi2X5eFP5LK47fQNmJmwShBqiBFU6hUZdLgshbtrPhgDBz4fwEqMyWrJrALGVLz5TwRvbOGNI9DvGRaiOfDUcrBc+DMxc23WD/3mB5LN7XVMVSYsC6UkeQqH9h/Bvn17MDU1o52aLVWMJeElran00PK+nabiPe5WOhgE8pP+EINCFc+/chYvv/yyUpO0J60mHTDzsBV6yNu23Rn2OB6Uv1eO2RhyI0+aP4loPyq8J2Y8MJanY+KBfAnpc7LguJMW34f61jXdU9+140b0I0TJF/EDZIj/M+WbR67AxFBJDpbsvfyeDMrFKrKpIfbNVnDztddKEzDC6QtYoa9jzQqIVyszSIoVee6OM3Ac0nhjPooVRXhRorho1q4EKdvhUTYdqePYHBIW2vVg5Xz6H/4k6XaZ5aIt6WN1dVWkAuKvlCLaHbryzIpJUl18xIPOpOTFmlonamRgQJLL4eJmGy+9+KKcLg6e3mGzaYjPSK0ZlVrvsV1kYU+kN7ngI+ryWDWE/C7PiZvN4mJzZB5aOcGBJsfE3VKioSliYcMsjNvzEDZG/0aiMEdIi6SEQxHFUkVZQC4UVaS0U8YBGAqiV8jksmkUc1nMVSq45aaTgobTXpJLZyvoybLPo1IdY+2qqsRLltR1watCtEPdQeYGi9DLtoQ5hTJhgp4jXrcwL/UXf/RLSqdQCsx+GrbLeqSwlLcAACAASURBVGVKEFWFpQB366t5MzpYVD9cSEuRplApl5CvLqJXrOCVl7+K7Z1tT/dZxobCwCR/qGsuWDgY8RASHKFK9PAt8xYPZ7nrFLIeUlAABfprt7CyMoMBQ5mITp1HF5LOz47b43FPPDJc4dD1B8zpm2PFCSSOzs8TFqbJylcqUum5gvVqSWjC+kaUVIHgwHqqsFxI8zrsygGeLGXx7ne8HSxl5D1VvizqtFWrBpUrtJIxTswkBMxqxY6SeOcAmh/i0qy/8dmiPs1dFqR+4xd+ILHuOlbiQlBBXQdy5FSToGDeLKmzQqpUOG/0YpHbvc0EXaFBfhKl/dfiqYc/j3q7hW6LjpgJCz9HDjZBei6MFtE5zrHrAgkL7jYHH4BNCIF2WYQXopsx+LTnlKOUIZ7kxQgeesX1YyG/NpwLTRM73cIWCwNDy1CdcxMYPFxEkiNzp4wkYzufQsD38FqCdj3lmvI0roiVFM52C1tXL+H2G6/DO9/5Ts/W2diJZ/Mlb97JFRKUsZKrCKtIkmDVjsHYHoV4XxjLqRv3PIAcRQS/9cs/rG1n5D9ic27nvPoiiuRMzbgO99KfiANbrR0MhxnsP/12/N3f/SUyDnZQOxiNyJiTzDoZB4w/m80Sb83VdYRtob7DBsm++w4Zt62pUH9qCUVfg8O3/HHs4PAFIqQLJ2/cRxjH2GMMDKG0WxyNE1qo3LLVUTHTx8RPJl9Chg4se9Kwhj2VQb1hiR9OGGu4FF4hjXTSQ7NeR7u2iU5tE//ym78JJ48ftbptItxO+DAGi5mRICMGrs4oRxx4gkwwGFUl6iRDiMpkcxuVNJFdUzLlv37wP2ixVZfsZD05JE67FewmgMOACM5vgP02EH4uwczR2/DYc1/F6tIr9neVsUTLJ7NrDCcaDcKmJDdSEMx+M24OdR12VWqIVZNy4v7/VYzane5lWu2MIUtc7FDX4Wz972x0/C7s9bizpmuz84SXB+k6LlhRCWI8vDzSuRISpRfJiSvK8TThNAezXGE+voE+bWmvo2Cwtn4VrfqWHLef+g8/aowez9eP8geROxBl2KBYsW2UhevLUMlNUbxOyNXyF7wW7z1OqwoMI/WhX/mhJBZUgIX3BIv6qmBXWALe0pPuH5tXyf+dFvLH34L7P/a3SIYNDZxMC8F3TMnxMwJDDPK02m4Lk0wN79rmcFSsPHfXWePYYkxRQWnjME63TJbHcKGmww+I3bp7bbNv8dz83jJ4RpDQriSvzZEv+QxU105CMNvpoU62YOYuV0A6V0QhVxSIwQVniljz0++jTnIGG24NE2ytLmN7ZxXpwRA/+1M/6R0d6MgydUmVbpskiBARchl2bhiZxeduucliCQfWKckjs0aNOCTjN4/Ub/3iv08YQrCaIfhhu2GPYa8RAoUDZ5JvO55aodnroDZ5E557+CHUayvyUoOcR+FhJ0LtdudHEVMW0N8xcgFDMKk6955t4i15Eeo7FkEL57zvWLyAH9NZW0Q5bWMtu8a97XD2wqEZQZtj8Kny7EwFEqgcYdVWshTqn0V0NqHuw5C/njMiZrqQQy5rxREZr4ztscojGQgf315dRr2xjnwqg//4Yz/ila1dLSQXJgoNZJfFErW+K9FKLNp1EBs3pMyRNufnGZpsXj2/mgYGUh/8T9+nKk5WPoSBskm3zJDZM8szx1dzZAylYrhEqtLmxLV49itfRLOxpsExqWDCYzsyYL4g9wVRn5+ntgjnKHZbnoUEASOSOapWGUZb4kv23MEVLTpBBu4cx8/HwZH4Pr4K2Bgj/MeCh6NmKt18F4Ieso8Ou45/TuPwWD6XLig0Yx6/n5D4UGLnS5RLJEZah0JmyQrZNDZXCRevo5jJ4Sd++AcdLbPuipayNAdTIIwDMOGoKUHkfsS4mQptFlrMwBbWirtW5dxxsWUPnPX5tZ5qEP/dr3fyn4Hz2o3suNDpY/KGd+Lxzz+AixdeRNY9VO5wMk0M6SJD1CoUgjhnHja9cgM1DB40ocupoJBCZa42Q6qAT0cPOQb6K+4nNjDWqoPPFQscKjoctPHnDOctBM5UqAmVFbfbDhnVTHmZrqIRvx93eIoOWybHDJChXKRZFyc1hiafvdVGIZfG9toyavUNlHJ5/NSP/ahrNIIO1Epm7zkHyi94nbnh6bYfd5MlZsi4uagNhNx5HkB22pHMqC9P/ebPvz/hgKluwhGKna3p9fAodpOBdmzlZIxKJgJanT5Ofv2343P/9ABeefZRZNJUw6wVtvJdAhGhsg0T52TKuzDKMLsVhN11hEwqyEOvcDYi2c8HkkMXjXr4wKL5WLw5WgDPzH2tGh/f9eO7elfr2K6WgIAolJVARdGinM+BJzBYo6XSHysglLOWNgHJ5stC3bhjudDKQPXbqG2to1nbUi79R37g+1+jrYLepDVx51g5ctcsMUYrLdrtLxsmRqGqGEAUxF1QSprhN37ue9VAx+LBcFJMYsxT3m2foR3mHYXDzhK9ajVauO6d34Gnn3gWzz/xJXQ77NhgHuHkpBXDGxZuVRoR+1kmJ6V8dixQ5K3lhHmMKiKe57HNSfOiAW8UQGecjk/kt83W72a75FX/bwraQ+XLprmDE9/H5JFLxvdxh4emkJD3jDOnZxqShWPv0SKl89o8SOeQVTtN443xvflsVqyXTquOublZfO93faelI51PF4Idv4tx8e/jYwuTE8JhPpDVltNB5L2ClxDzl/qVD/w7lexavbEjVGNNVqN6kQ8RN+CFFhYWwBYQxWIeSSaHzuQJnLu8ise/8KAexpy6IeYXZ71wwOyWhVKmqqimVNM84lPvdn+IQgOOje0raYMCD4/sFheedj0ctkhphoqORY5F3Q0jvZPDGGWY4+JzRQgY6jBaXkdnhQA4ct5zRmgZm+8RIVSM7w1o046sSWPSnzVGSqrLxj/b4udff/11+OEf/EFfbGO2hJNq/lHAqJ5p9HZlaTmHDDONYxa1cdS6mltH56h9ogpUc/BLP/OdymczbolYkzsnVGXknMnbYq8RPvSo1ssTCCwZquX24NIO8MTnP4Mrly+OgILyBInwjEENFQpEzXZL3hrTpq2nWBD+xu1sOGJmUkIhW2Jf2ACT/DExY4iZdp+XvgYuEJM5vtPDHkc0EL5DaAIrKjRGy8jR89BHvVy8dZeySwlZKabOuU4K1cQxy6g0R/dXjqAuuPRd73o3/vk3vHdMjTMnb+2/FPJGaOpOqXnf5mkr7aww2Xh9Rllwe27fjHiC8WypX/zpf5swSJeKYTG351S5uATuc85bjpCF8bEe2u1jmlNNzzFVwvnuNB556LO48NWXkMomyInUDiwszo2AFAvx0t5vu6ydHdpDu9ix8NiNoY7DpBAXd1/JAIxUImGx1N5uY55Q5fE1JinEJa7Pn2PXCuN3vH40qeS5ec45FtxqoS29Glg2+WEquqcL7tGCqWAjTrCXaTTwEVU6ncKHPvQhlUiHmRPbhw7pWBp2V0CtBp73NQ3rFC0nMHCiJdzeL2a0+B45aSwf+In/OyFXiv27SbpXB6IRMS9tOLSyLN7wLpIQUYutBu9ZdIcJznXm8ORXHsa5l55Ft99GOrHWUlNTE1LZFDcurrzMPqE9a0jL3msGtJiHHwAHB8hdoqY3rE5UV0Dz3G3X7qpxg3stsRI7OhY6zAavN55wGXfUYnF31WhMqoFIRtm1/IBSvS41I+dJZLY0uh0nGoYdbvdUkkP1ru5L0XigVMQHP/hBoYCGVnr1ihMTuKjGOHGKkYeD+tmTM0ZiMAatSIteVGkIk7FUhcwpu5hC6o9/9/9J1HzVS2eEgdDekBJM58JPGMhmmOVJI3EUiQsshIv9vAg2II2vrnbxwvPP4qlHviSCvvBqVmeW2LzVPPKYVLOPhhoV8+wRYrxyld96OBOLEwLAWnH+jTtZsbtHBru7w9E9j+3Gw6zxRRy/7tdqgLh3CA0xcj4rd4xahgRI4YsgJ4222Om84deElookje1QFjQaF+/EyWvwH37sx91OBxXZulOpfwrDWmbt1FLL1HIIp1KqhRyGHWeiOOql4zjU9M+aBFohgiGRCls/9td/mBTLRWTUSwQCBZKEKTfr2zGi73oFQ3qw60QpNEmxwRtj3DSu1od48atn8ehDD2B1ZWmUiy6W8ihPGJPFvHEvuAtb64sbPkOYknEHSw/oD0xvM4SGYyTGzOvGZHxtDB3OllKKXgfN7yMBIgFyGz+uBew6VuhOSFRC5zy34I0x2aNIIW190MI+mgOaRTIIO2u5ezstIY1f//VfwczU9AhsspbfFs4JKQvbzHvGbg/AhbaakYznrpW/GrP1u2RM3ziujVMPff5+IX9q0KL2y757vGwm3H2Lei0nPY4hy6HxdFo/yeHxVy7jSw/8Iy6++qKpmEwa+VxWhQfRp4XccF5OdUjFDLpt6xca6pkTHs1aaU85iVTz47tw3KabJTPHJUKRWPiv1RKx2/lc4/cct7OKSZ0gEOxPYeXBb1NDH2eQuhYZjzLsnhmFWeY505QbCklG7Xd/93fjDW94nXPw9FcRMGge4h7RrYmXFzVpnA3rfPQe07DUKS64chIpcKo5G8rsGcnRk1kPP/JgQk/R0pykYxqYMALhnWLbb1uXWz6keeNx8k5KD8JS3VyuhOcuruIrX3wQLz39+AgUoNQyfjS8mXnznpAhkeDTAyR9CxnGqzPi4aJOy0AZE7RQw5EsYYO+r0XG4vOhHcIPCDX7tSp+3L6H4IzfS8wVz+Pzmv2ehakhMCEs0cFR3HkdTZHHgYMH8KZ77sGdd95h+RWRRUwTRe6BZkkOn0cQ0UslFt9Ewtil9PLDWbOMJVG0XWbqeMtt81E8qfT5z9+fsBMv7aHVPRmfigNSAl0XIqmcRXQseLOeXqxgZH5a2DbhTZ2pUcCVtW18+nOfw/NPPKLUpXUpsm75LMfhBLJVRKdjvcJZE8XidoUT8jDNQYtJCE95F3TZ7T8mQqEcOscH8plRV4TAv3fBEXOc+IpESahsmYgxtC3MQGiPuHcsfpiC2P1a9HYfe/fuxfu///2iHhsM5Pdy+rAEMG3PZxTh3TGxr7uIEuwU6Y3reV+WRRlgYk2AeS91qnAiYtC2rJWJbRoCQcIlIivorcVSD372kwmzVjqRJ2vdh1l7FQDEoGt4axSuST2pgsT7blLd+SEtjDFT6QKefOUM7v/E36Fe2xoxIwnAWO/SrOq2u11SZ62WizaXLzEyHXCJiYoJjh0+PtFy1EZJGh65YDZzHIXiIkZIFRBo7HK+N8xULGjYXA1ojIgYAjCeJ45dd8cdd+DffNu3e67AKjZpQ6PG21SpF+2JXGmYugmZVW8QhwgnkjtcvD0nDHLhtHO9k4L5GAyTdxeVi22JKzp0Rhahn0EBoGoX+vfpf/ibJM3QqdPWLstn85icncYLzz6FYcIwjJBnFXv37ZHtaNU3MUgySGVYrZlHZgDkK2wIYwxPqphXlrfw9x/9G6wuLwlDZ5E4ww+q6Xqt7g3r2BfNeoMOKInOlFEI70kRIy8ECXG3VktxtZzH6LliNnZ0ksAYOTGw5JjIWAC+N6jIdoSUYf29riF8/G9CbdpGCQ5f/NAEHCfr2n7mJ39KY2ZhgHqjD/qqTbfEhqVbWYynpvYD48rzFa1GuLBEIlUbzoZ9Y3kBnVDk7SrDbBCNMzqxaYg0mUHhs+ikBeMPcvz0j4zFk0Lqr/78D5Lq9Ax63bYkgdX611x7Eg/d/wkcP3EKi/sO4+WXX0Q+m8aBw0fx8tOP4/ipm3DxygomJyZw6dXnkJ+YQc/JJCwiT+XzuLzVwSMPfUYdE4kzVCtV84QdoCB0yvBASJDiCqtdGn+Zat/9XahNBXoKKSJDZHlmkiNjUUMtj9vmXe+eMazVnekeHpoY08N7sPjC8prjsWqo0sgw/b8/87OYqU6pw7HUvldi8Hk4FoavfFajEVGT2PtCg9gzMS9hVCRRmdzzj0NtKDChUaTxmPpVBMDuzz2rvuUpB+xVquY6lofv+r34GYFVH/nw/0hm5mbVe2t6egoXzp3DnXe/Dl/8p0+qo++RU7dgmcXvVy/h+tN34IXnnsDJ625Coz3EwsIcHn3gozhx+s0oqEVFHfv278fTX7of5cM34S8+/GEsXVpCPp9RO6geC/ac6cLJ4aFkQnpiQcc93rGFJl4VvTsNVCHQE0wWS4wYkGKCQVNjDppXcnqXYOamJQyBKbN6xc/90G7lzus6Bz1Sq9EiOrEMHR1F64OSYHJqGj/3sz+npEh446ERgnI1KgOWX8IerB3tYIJNpkms0Q0PYlPNupMuIoyjsLIxACneuXzBKkM8VCQMbfQuo25Rm/R40kGpKN+l06xbXThbpdCGs/PC3MI8dra3MT+/gLOvfhU3n74Vzz/5KNqNbVx7+xsx7PZx5sUnceTkDUpyFEtVzC4eQnlyAk9+7mOYmN2L/Ueu02IfO3YUjz7wcUzuO4LOsICP/t1HUaMq8dZV9DKFJMkeGUU2asis04QdTmbVIl5HNebIjHunEarJ3ku1pcSQMTVoFY2aPDXX3c1ta4d7VYWS+4RMM1YjxYlnSMjvdz16i5F5P3rXFk7mVaX5rne+Gwf37hsldsLBJFeNY1LbixZPTjCba9i4naQQfk803+NX7sDwJaiGubhsTBC+C7/yOjqZIA1t0si9B6N0e3vHyCNk/uq4Spbx9pD664/8fjIzO6u2FWxNwSTG8ZPX4crFC1i7/CoOXH8bFucW8NzjX0B5eg6TlUnUG01cc/I00rkMnvvypzTA46ffpAXau/8AXnziATRrNRw59UbMLsxic2MLTz76EL789BksXb6sXWGevrMynMkSB4lG191oWZl4q0h+jhQqPgiPfeAujxYUVu/sPcZGoIsd8Cq1SJUfdc1OiJQqde+fAIXh60Md+CoMWiR9o/bypTiYcbP4vEAubQ1riO2Hz3H06FHccMONygqye1TUG/EZFNuzOW+vp13ISwVMSgRRi+LnpfCrteMsqgcMhZj1d1w0CZu34OTOpkIzSDnB7MysasXYnSoO4su62Uj99V/+j4TF6LWdOqqTVaxeXcbhoyewvbmGK2efw+yBa3H0+LV48ckvoj8E9u87iq3aNvYdOI7iRBlfffJzaOxs4/ANd6HEHT87iwuvPouNy69i7vAp7D98rR7wxScfwKByAB/72Mdw+fKyqb2BdTgO+0Xpj7CEoQapwnzIyLZx8Ny1Ukm0/Q5YyJN2gbFsmLXVjOI4LZYxHV6T16ZajyTQbjLFD5rLG7NVbBSP7y0c9DCR2kQcNW8G7zn3cNCII3CcLHZg/7SJsp1lwrCM5nHYbSmKoa9jdKs0+sMu7Y4EgYe55Qs2N9T/1g/V6r7Y+ULOGokjjZqKKNVpiTVfbPbXrKPJDlM6Xbfgba0HSP35n/5uwqpEa59cBM+Xmp1flId86ZXnUJpawPEbbsH5l55Rw/mFPYfEpZqc2YuFxUWce/ExbK1cxsTiMezZd1iLvXzxPNYvP4t0YQLX3vI2dSB89bkvoNnq4vMvLeP5xx8fqR9BmNHPVOwV271c5JKfFMDfaZFzu0kaIWV+Qq86D3i2R4APTxQKh8lLYwngMOHCtKrRjiyhEWaBqcoAddQtSr3COXF2hgfbVZl9NB+DZT8sMOQiqZuTzibxhgEOdFBQeF/ZVPfCC/kSDh44iONH9mNl+SoOHTupnnArK1dRmShhdfmiHK3DR67BytUVnXaYKxZVhdlt1sVJLzAbmStg2GubZnNIt1CqamytTgvVShkNP6lPWolz9Vd/9jtJvkxyoDVutzjVmrGtXDwnZujJG2/F8tIFbK0sY2ZxrwSjOr2gU/GuXjqLnaUzQLGKhYPXYnZ2Adubq1h69REMBykcOf1mdUQ899LjaO9sYjs7j4985K9Q11FN5pUyZOFXWtp9+/Yr3hYzxI8nZlTGn6lo1ZMz2l97VaaFFlSnFk7xWlJvcaY2QaOx46oihqeaFN3XF5+2UPdxhzHUvFKq7jCypo0aYZzUEeDLOFizGzNb7xQV5jmGoNjeyZgEnt56772YmpyS8DY2LmNicg7XnLwJly+fxc76KvYcPIyt1VVkEx4ydxUz+49jbn4R68vn0ajtoFouQIfjFLhBymh3Gug0a+i1TdAIdnE+Un/xJ/8lId+Z+LUC+X5f9pDhQH19BcNUGvsOn1B/tPUrl5EpltUMNpUpYe/ePdhYX8ba2efFtZo7eB0W9hzAsN/Buee/qCMo9p28HYcOn8CVSy9j+/IZJOVF/PnH78eFM+fQ7Rnezfvu3bcfh09ci/m5eeRy1sEvuv30O9bnrMQDYZx2LBXrP3Px5HQZqXrk8Qu8oPCy+I5xrjea5zPy89FFOECX8URKNKoNgYmkCSnBStHGkY9RPDiWw+Z4IlY3xGs3JByhdrLhPF/T4F8ybCmQxw7OYX7vIdz9unuwvrKEKxfPYe+hw6htbKDb3NKc7T16E0rVKVw5/zLQazGzquKLfGUGM/OL2NlclZlg10rejzSpEos1//T3fzkR31nF3XYqnzrRF/LoNJuC6fbsPyJbsaZMFoeWRbZYxsL8HkFzK+eeV0gxufcYFvcfE3l96dXHsbO5ganFAzh6/BbU6ptYeuUZtb185lIT93/606jvbKDR6eOHfuKnUW8P0B9aX/B+t62meYwfCXiwebwWiIiR0CnGqhazdhjX09apM7E1j+VxVRFeqcpFaUMrciAwRE1g6VaDaMPTDR5XcMnioNnIkAmNU7WqMWIDsKHNpcPJ8NLOFfXTdrx8KFp18/ddnnnqfcfl7XtmXGeSqZdMTxSmQwcP4Z7X3Yna5oaAm15vRwvOse+95laZ3NrmEmqbV9H1as7yzF6kszwQponWzgpSgz62eYpvZRKTc3uQ+uPf+/kknS2gQM/RWQ18eC5Kp832WAkmpxcUpNNpo//KTZUrTmDf3gMCA66cfQHDfhPpyjwOHL4OxXwJaxdfwtrVcyhOT+PaU2/ULl8+/6zUYbtyBL/727+NlbU1fNcP/LjKaLa260ilzYwQwKF3WSa/LUlEqqCw8RpimGZJY2L/MaYQ+xh2efRCH722N9cbU8uWGrXr2kIbYNwmsqdG+EaJChiWX62Az1pYRIYvgI02QxgnSQaiJWqSw7KMcdXbTYV90aXJEiZ23rbF/vZ9HMhqHRSkPVRTwTH1UC0V8N6vvw95HajXQnNnW4zUvcdulTlbXzmP+tZVdFtNadvS9B6Z1+3NDaBXw9ryZWvik6RQnV1E6g9/62cSNpnLuo1MeUaF8KBaMOoQlylkeUh3r42GmCZZtdCYmJyRyqfdbuysI5cvYe/hU4JXV69exOblV8XeYAjGU9uvnHse9Z1VzB64Dn/2N5/EiVM3Y3pxn45n1IEvLEFVKGPg/wghEzrURSGbt3M1szxkhXGmgShpgjE89LxnXYLZs7TXZN6YkGRXNdGKad37p9dPDRKN9tSvLE+wYjCCcFlxysW26CCl7gahBfg7zoslM6xsmDvbnD5r6MfFEA7gvcKjC4Oa0PF0AF7DY2p+r2ILfc5r5HrWFLA6kcc3vOPt6LcaGPa7SJcncOyaWzBIp7B+5Ry2rlxgcY5M4fzB61EqTmCYdFDbWMba1SWFqRSwyvQCUn/wwf+YkKhAiaItYvsIhhNsXqf2Dil6x1UZeXYopoqU9BdLKFen5KVurS+hV6/JBMzuP475hUX1DVu/8JIWYM+J27G4cABXzjyPVnML5YlpPLvcRXlmDp2etd8S89QXkhk224l+aqA7TMzMyXazl6p77oasWSUoEyqceDaHS3kbCi4YPVnZzYT/DeumqdFB65HedWKAWlzJy/YjLbwgYChTMlCOOrSAOYK77BtpAbD7RFvevPkJ1pGY17TkhrUXCdqQBMd9iPBfDDJmVScPaAW+5Rvfi/SgZ+ZtagYHDl6PHoZYv3IejbUr6LGWPJNBdeGYmgT3ei1sXL2IAR01xuoTFZSn5pD6g1/70YROGNtIkFrERVZK06sp1JvDKx0M+7W0W5LKYnJ6CplcEd1WDTsbqzqFoDp/AAcOHlEP1NXzz7PfFqb2X4vZvfuxvXYVm8vn1PZyYt9NuLTdwOb6ttAuJUl27LhFmgp77Ta5s7DL6sO5s4lghSMU5bWMyyWILhQcL71QCpESFd6ey0piTCtQGFhTpSMn/WgK4eXMoHmKUhAoETcJgZU80RsPx5Dawzh1LHw0UkR49LxnOHcBgYawBFrGnyk00gxjPVzlHWWzeM+9b0C1lLPqmvwk9h44KlOyevkVNLau2rNkM6jOHQZDO4ZrO5uX0anXrCd8Lo+JyWmk/tsvfH/CKgZCRTlWIFKUrNLLzqygM5GyKkURERkzisGWQ5GdFgoTGPSaaNW20Go0QCeBi02MdvX8CwoBJhaO4NCx42g2a1i9+AobV6By4HpcqvWwvr5lZaaqELWJ4iIrJednafG+ERLxIQmSiEbknCum9Pi5qNfm7jOWqhMTiaDpyGg7tkH88yGUk9fnlIywMLA7sG4S2ZQVshMjUNJDXYzICvW0qHvhhoFbXpq7qOskD2kYp2AFeV+dFb6mTCcSKiGMwaAJX4Ff3/2W12P/4qzWZXrxKKbmFiVcq5dfRae2au23CnlMzh9BuWTtvzdWz4JUETmZ6Swq0zNIfeg/fXcigqHjyAmbzbK7AltLyzYzCc4qA3c2VFCQIJPn+ZhF2XpOXmN7045xqlaxsO+ornHlwsvoNtaQKc7iwPEbJCjrV86i3+mjtHgMm/2iuFRXr1wxRMhPD7BeXl0hZOEpR1ZMRx555YUQLSpELz5Uk9eoBGU9eJ4q11RmxOKWnuTCkCnCyfDzNpyDprM0WJbkvdA73ThegpSfFnLUbqQww05D4PUUQXS6fta3lSSHLQ8nLnZ34O2RJo0jKFyVuYDasVFxxOV77nsD9sxO6muDMwAAIABJREFUSkUX5w5g3+IBLeLm1bOobSxZGXRviPk9R1GZmsH21ibQ21I0pANwGx39PvVbP/sd1AFyoDgwNokXu8MdDJaeplM5JDnLVVN9m9NCmnAJ7A+mZCNVx9YWUrk8Fg8eEzy4fPEVNLeuIElP4NgN7kEunUW31UV25iBa2WnVSa0sL2uRGA9zt6lGKTPEsD806JBN5ssT4IlEskHecC8otOwWQc+a0Kd2ijxj8uDN+7bOidYWK5L+dK7YYpMTpaSHs2aiSWyUNxGv5vENwx6dKPY86arUNpoXtPtdMw/eKIj4dajigIEjPx8xdhAX6DyFoxhCbQ1sR2WaEuy3vek2LXapNIGpfddgbnpBuYzNlbMYtLcUmRQmJjE1sx/FiSo67SZWll5B3rVVNlfEgIWHH/rAdyZiOaQtO5RmGwmiUZ6xIQKsGmVWJqZTVmzOXaiOPEWUJspuuwaob22LZTo9u4Dq3CK21y6jvrksFHnx0CmUKhWsXTmPZn0HufIc2qX9SkRs7WwpyU71yyOQAokKtRyn+ubyhosTdaKNJVOTqUL5QGOlM2Ez6UOojIZwqx+uqkn1BjTMGFEzWJ8XClZeuLLial88xqqETOkEqTmfU5iUVnXnyrxpO4SdziCzXJEAEVbujFad3R1HZYjM4Od8e8M6TmQc16gx+CE0//xdb0KF53snKew7dBIL83sl1Mvnn0ONNps59HQWE7P7VRde21lDNunIBxLUW5kStzD1X372OxOzOVb0zZBLaFTBHDX2CleaMLFQQkcTqNk5Y/Gy7IF1sx+q9zYHWChXMLfvIHrNbaxcflU2ZfHIDZiZWcT2+pL6irAJfXfqGvkKXGweDcFqTsbtUaHoLbSlVjmZhFE5JmLcUc9katGQNf7nwgX9iMQJ29nBJPXKEYV5u6fvMU896HfkeCrP7nGwbDeb1PJ0wFJeKBfrzsLDVt83liA7kKJkhjtYTGTQOYquhMYPYzLeqFfRwcJy7pGPtwaC8iGcEcr+qd/yjW9DliatWMb8PvO4eZrP1sqrqG+tWPuNdA5z+46qgrTZ2EK7tqbjP3QC4YB14hWkfutnvt11hpXQBhtEh6MzvFExALnZWaTzVn8sJiSTD7Tn5K3xZKC8nYqrcy1KE5if36sdtXb5FbFVJvccxszcgjr4s3mMSIvlEwpVOmxDUa/LuYlcbuDVlvWx8ETd/dkf1Q84CcZKwkXgJDsi1uq27TQgr57kLlVhuoTaGTHe2sPOv+buMz67cs6eCrW4Oiv8nCRJOX19rzrReR5RgUJBs8pSMkeiEQl3KtOl7CYch89F01i69jI3znc3X4MttqzDAgWHWmeyMoH3vO1OTFan0RoMcejoKVQmJrFT28L60lfR7zYFnKTSZWlT9UEb9pB0G1hauiRNUixPYDhII/WbP/2vTY37ohqldRdW1NmWKo/M0OCpFFUYsnho1geMks42URaCMITIozI5h8rkJJbOP492s4nKwkHMzC5qR+6sLVviYvpa9NgxMWV8rJ4X64fHysmXSiY1iBAn04I6e9MSGNwd3Fl0jnhdlsFGaSwFNc77oAqLuF2qUud/GeOFcTX/RuFmbRuJAqq58lBqBIl6fM2TiMPmmrnY7aYcp/Ba41w3LXQO++yVZJTrqLSMggdreGMLLSrx6IjqtDTD1FQV/8c736S5nZxbxNTsfoVXPDu7sXEJnXZNglyd2oPK7KLYNIxqCKrwpGSmr3fqdZRLk9zZ36Fi/MjcREDPiVD44+CCtX5iC1s/c1pnhDA+ZjuJtJrCMUHP9BxDNoIwk/ML2GKXgc01ZAtF7D10UiqPP7MNZmX/ddjqG57MhHuj6Uc9DW0RR6GKdiorTzpIuEu7hpUTEVP7KLbS9J7oXLxI6PBZomCdpkjtuHg3jdvqrWk+goIbTQLkoHq7jvGwyey9dX7UGVrcJN4dOUgQ/MoIYLz/anjaUZAoCpXrU+5sgwGN2B9IG1uAc17vufs0juxbtM2RLePwsetFaNje2cTm1XPotWqoN9uYXdiPdHZCm6DXb2NjdUmhqDUw4Jrlkfq1n/y/VJ8ttTFWlmq4MGucrMsfU53y1kX5zWHo3QJ1oEqprF1ON39re0tYNosGipOzysisLZ1DtlDC/P6junnS62Fnex2Ti4exmSygM+Ahbzy1hhMPdFpNLabSrCsrQsbUUbHfwvbahtSikKiehU089ti47XZS4Hi1pdGS/MSByIJleaotbbkVHhi4stulwPhscYCLV0+6lpFH7WQ/2d047H3sFEE7etF4YSE0VmCw26dVrFvaZTpq6pC4W8BHLcCzWk7fcho3nziMTqsmBK5QncUij+FImGhpY3PlPHrNGjvJoDqziInKnO7RaO6g19rRQQHUVKRIsX9b6hd+9F8RNbbzPoTC++GnnguWeo/KSTVbpUfMHizehsIPbGOF8GR1Uk1pq1PTlldOpTAzN4+rF8+jN+xg76HrpHImiadfWcLk7CLWM3tF9WFMScePue0aKTU6M2tTCRFmgsjk5RENje0dqXvBlElw2g1vHq9uDApSLLx2ZZza5+UycVipOh6JyMIODFGf6ScI+yLuxskegqrbgrFbuctD3ZN9kuJCC//uW6/vsb7qTGqIaDFioBikGqzVfDaDt977Nhw5ehS5BNjavKjsI9X9/IETmJyeQ2o4lBrfuHpOY6YWzZd4tGNFgkuKdrOxiWG3Y4fJcjMih9Sbbj2U3H76JuxZnEW5wGMgbGcYsmTHOUnL+JlVVNuSfB4xIftt8CV42MpE2equqxXtNDam3X/oEFaXltDpt7D/AFG0JiqTU9hcX0OhmMdw6jp0kBOjIzhZdNSIVtG2Moxpt5totWroNNtqkcm/G1drt8JDp+xSCBMoHAv4MXaptFLWIFYdqRB9x7UQdppwf2AkiqhBD7ttTiNtOyfDW2RFoTyv56Wz0jKEPcWMTsk5ox7ghomW21UeLyV2ib2OHz2Kd73rnTrakX7H8089La0wOTcrz7+2eRk7W5tqaLD/6CkU6FUnJG3WsL58Fjwsjru2VJkBUkZy5GIPBy0Mve1GVwfDVZC65YYDyc52DZ1uH3vnp7BvYdKci2Qg7teeuTmxKKpVghpMORpRwFgtwqasFbPjuJwoeucKHZIheEYlJW91dQULe/ag3e6iPDktQiL9vurCYaxiHgl3sLJUHaUtZZO7jFlbaDUbqO1s6G+M5UmOCOyZE0Shi1NpFaOn2bynjEabJTNZxc/WoZ+JClOlPG6AgsoiCNavjRIgsJpoU+27rUWCjCDVOxiiFGd48z00H96TLCNUz2JrhWR+AnAqm0elmMVEtYiDC3tx/fU36Pip8ClUxpMCnnj0EQlloVpFv9XC1tplgGeDF4ooLxwWKbRR20aztYN2bUtzRH8qW6yiVK7aCcHtJrrtJhKCQATApE2ySH3vv7o3YTqvR8eDXYa9+ZyqCr0/mb7qRAErLdGBLf2hFnl6ahJ79u7RQSqGaLGSgtUQrGe2Qv04TqJa5Yl5fRQqVSFOxL6LE5PoVo+h1UuBNWeKibsdLQ4dL8boGxtrGrg87xbP/zLcOcJEqWOPkYm4EeUSEZD1awXrrM+QjQfAqgyHKFjBCIUsT2ZhgEgDNGEeOAU3OxbZ4E1r0MvPTfL0PyJnLhhWnsPr28HqFMZKtYo98wuyvRN54hCb6LR64gIUJmZxww03jLo+EKmjKfvyF76AieokSpOTWuy15fNqbstoZ/bQtfrabtaxvrGiEJbRMdkz1akF7XpD69qq8GFYxnFIjdP3+vkf+iZtEjZmV6rNCXW0wZwk4b7qprRbtald5z1MlaPyqg4V+fnpPTOzM7j2uuvEqCAIYIOwDj4E7SNVqQashTkkU0f1WcbqFBR+JQOD8XOzuY1+u6OfyaYUB9pP9RXgIgDD2leJBOAn7vCe6YxVTPa7BF94CkBJlaOBgKnvJ59HqVbadfNfmC3Ty7NbnFUlJzy2Vh8G92tYp8Wdye4Kx48dU/NZ1p2RYXLoyDVoNxs498LjSPptEGsvTC6iNDGtkwXjUHoWPfL5udiV6pTCrPWVZdRWz9uclWew9+Bx45HvbIrlQ4iaY2r3eiiXp1Am7yCblT3vd5mOrqtdds6Zralf+YlvVehFhUz4Ubli5oVVAdGjhTJnw20UmV4CKFxN8fd2Gp1liSIG5c6k/TLbbwT9bsfO/5pfXJQ22L9/vzx3kh6Ge06LVkumZiQSqKLIrWq0ttDheZs847vZsF2tQ8GNzMAXcXsKJl+BSRND77Pdh0jypFsVBcwwNOFY5ZiNjk00Z288V82Ja+zU7JgI1rn5ATlk41II+PXUtdfhmmuuwebWGmZn5zAxUcX66jIaNfLF+rjx1rtECrx85ln0W3XNyfz+48gVyzh06JA0DL3xKGp89OGH1fF4Ye9BXL54Dq3NS1aDXZzGgaMnNY9rq8syZdnUAM1GU2dwZrLkBvoZpMOekk6N+rZiciat5KP815//ziSqIuwQUivoppo2NTeCeXczSqPOu+pY7b834ELagQkJP/vLSkkNmaOU8e+0pXSoKCjqMcJMenU/7nnft6Pf2UGjZWgWsd3hsCe8emdjw8kTLQmWtWvmrjWP02yxOZb8T4I+zzmhGTFP2QiJKrLzDglBPxpRguh3iOPmJ+QxqZKy9GppghqqjLfde69ds83zQbMoVytaTFasVqozow5Q3HV0Lq+/5Q70Wh1x6evbV6U5D5+4VZNPPjmdVDsdyMptv/DQQ5jU4Xd7sbWxgtrVc6i1apicP6bUMcda49mpTXaeaongQLw+V54VtVspzWSI7Y2r5tekmYqeMELGf/9F9kET3OMkPe/d4VxsoWVaLMNwhdCovYNpOU2hkhCEuaPO2tpRmJPDybfLqwGxeox6aa4awQzVpyWXTuPU130LtjpsoleX3SNEyd5xW5tb2FhdQTLoOH5uxEIuaqdDLNwiAnnebPQeDVr7xLG9/4rCoYHIlJEGDWhW2pr0q4nyqE6d5ufmm2/GwX3k0PdF0ZXjxRMH+fBeU85Qi1jC6soVHSBPUn5UuzS3N3HkhtO4dPY8Bt06NtcuCTy68dZ7sF3bxpEjR3RSImFTWhCO60uf/zymZuYwNbuIrY1VbC29it6wh5m9J7Bn7wHVfK1dPS+NOzs3g1aTMHMH+cqsauTps2ysr6K5sy56mBrv8Yhp+kh/8ts/4H3QbCFUye8Hh9mC+lGAYyfDKhRLeeMcnbgzVP438F1CjwJivGVlnE1l8pSo97ZMgxPuGPqo9CYzgeqJN2qhGVq0CBgM+qpDI6mOtCjmzDfW1zA7M6NDaKKihF2XVP/k7TEMJCGyV1S8ywklXYgPTRvLF0/lLZQKKGSyuPGGG/Du9/4LhXWdTl0EfkPlGBV0lQ3kiwwcqnU+Kz1fmbp0GitLlzC7Z49OGZC6L2Rx9cJFXHPtdVheXkKqR422g6Tfwb6jp2RCWFBRLtuYTY0n+MKDn8P0zCIq07No19ewdO6ryoQdPH6bPPJOc0sHwHaHwPTstNLK/V4TufIMZmfmNa619avi3ak8macPq8Chi9SHf+dHRottIZf3J1HHwziT2k5mGLEhBe0ZnCreGp0kPyhUjEo/RMXAA5oDU+8Ww6Z1noaYrN7OcgSqDFNo5efQyS+g2W6g120pxqYd7zQaaDV3pKZ6ZL2y1kq4vbVfZm7aTtyzXR4ghQANP6ScEOTMzDTWV1clnG99y73Yu3efaYheG7fd9WbVk3OxL1+8LEHrdpog/6xcrSppEW1G5Cc455sTWd/awMziohaRqrY6VcXls2ex//BhrKxela/BoorlC6+iunAIczPzYHRSqfD4KFPj1C5c7AOHjomHT01QX19Gq0Ou+M2YmZ7FkjgCqyhVyRGfx/bGhnh9E9N7MDU5q8UmgsYTkzkHC3v3iU7FRj+pD3/oRxPtwniZiR21QTYQwc/zEp4ah5fa7uBLB6V6laPgVe+sFDndKGS3YwYtAxSokmBFaQ1ChoYuDZmTTU1iY7OJrfqmKE47m+tsrYB2py6An+8jt9zgyzTyaibIrhAFUW/Z8oKeN5242s46zp05o5OD5YB5XzPrMgS0egNcunwF/+67vwf33PMmdfl/5pmnMTc9qaggSn051kbdNAjPqpYvkIJUJ/GAyWpVOALHUSpTnW5gbnYaV5eXsdNo4Prrr7fvazu4/ba7jSY9wR7ljAKsCPHBBx/EqVM3YG1tXdy+2uaqophD192qg1fPnXkG2QSY2seESB61zW3UN1cxtecgZqbnVQ1y9fIl60RZLBnbKE50+JPf/qEkCgREY/VWjdEPk7syXsJ5/Sxt6/tlQqKe2+y0pNaNFAw/US96aXpvci66drtfUI4Z0SQ/F5rHJUl4vM3ygWtuxeKho3j2madw4eISVq5exZXlS3Lc1Bd1dhYnr70OxWwa1UpJMXJc3zh4ea8qoZcgN13OA3ciNYQa1w/TaPUH+PgnPoFbbrkD//7934/6zjr+/u8/gce+8iVzbPw4BjmTxKjzBfHv6E2fOHlCLBoVEKiYzzooMKTiTQnt8kU0jZWdWyR4qClRWTa7Up2wolB30D73uc/h5MnrsHR5SVU4w14T/e4A+07cjG69jo218/IbZvYfFBeP8DFbWk/M7cXePQews7OB2tam5fRlwzkHnpn72z/8aanxAOwjTKKaVk9MERVYrWidjvRSQsEWNGykcrFjjdnMsTPnbVxpWBtn7zzgxxf1ujxxqCTkSCfg+HX3n7wVB/YfRKu2jVy5irnFPejq8BlDuRhFMDR76cmnlOyQifAyXFtb4/AG6udDdxKenxDkDNLBMAfCive9412oba7ghWeexSuvvjRKDgk1pBZKLEMXzeLJsKEfEXRg3mNyakr2mKElNYyYs/W6wkzGv9RGrVYPr3vDG9SEiLmJhKnWYYJHHn3UBHYwRLtZUyODZquDI8euxfLlC+g2a3JoF/fvw8b6ppVZnz+Lyfm9mJmdx9raFW2GcnXaDnuX752oKDD18T/9Oc96xaLEQRu2IHTVY+G4+GKMyMZ46exoMQ0UiMW1isZd+dC1YrZdnYcNZ77ZeG86ZXOUATp43e2YmZlDu76NVg+45uRJk3T2YvF66VaziacfeUSTZbVc5L7HgY8mbAGt8jMqDBiZJdvsSln2SKIs4u4336MzPK5cvIiVlSVD8lhPXSAtyzo5jkwQixG8S6OlVXkd4tI0N9ZhgYJAweDPtPkkVcq5K07ge97/flxz5JhCKAI/HOcjX3kEO7UaSjyLs93E1GRF9fB0tLrNBiaKOVXDTs/PY3V1HYcPH8aV82dQnl4Qf2Dl6iWU8gVx0phfiDPAei0u9of/s+9sSyJwN5jjZd0LvARaDlks+rhaJy4rmk5sei/U293NVNbet2t0wIqfejvWEE622lmgUTZz9NQd4kqz9HRzcxu33nan6EN9LwgkiEsy4PNPPAHjjscZnS6oLm3xe9M+u2duywt2fjzbhPLnm+5+HTavXMH66gq2ttcFCAlhcx5ZtJuyyfImc+54RuPa2OWMAthjbhxyVeTC1hq9Pk6dvg33ft3XabcGBflXf/VXsb25hTvvuh0zs9PSIoRl2W2KHZwD++dYGT9rnaghU8DUzDQ2NjbF0WPju+iwVC6woH8LqU/+5S9rZ4fKDRUbReheyTc6fZ04ehh9U6XehMa98dHnojmNfm9N9ETrkZ0mxkwN63XVbvt1cLiK3kzLnLjpbhRLRXD38nD1O+96I5JhV8QH+ges/OA1n+VikxDo6dlx8zFuRsxRsVMLOOlW62VsWXK3KLQ33nU31i9dxubGGhrNbSUQQiEpDeu9xSJEDWaqJYeM/x5HJGqR3dkN4CoqRukLTc0v4r63fb2gz26jJkH8h099SpwAopTtVlPPvr29uUtXJmihA+ZSgqzvu+8+1Ld3UCiXlG2k+aht76hogI6q2Dre/Sn16b/6oGlXV8dsnRFVhoq7YWCFuFGOhu2abtsZHCQJDeEcGcgSoIqlEE2VxiEzpt9JXrTT4Omhs5uQdxvy9OO1N98tpIxNbzc2d3DrbXcDSR+dtpEWCMgQwHjpxedEpzWYNHaupSo5vjixwMa/Cxrp++iE3DcTdPr1r8fy+fOqH6cTx6DTHDM7mUDM20gWceGdzCAz5R0gomOSiIuuScRC8ffaGEijmcBb3v4eVXU0t9Z03ccefxy1Rt2Yq85eVX23OkuRjGnnoZHvTu4AfQGdlUrT0TUYuNu2UwtOnDgpp3Bxcd5qyD71l7+h0Mt2HA8xsSZpRKFMPXtxwKhPib1P6tDroQlUkJkSXXCDdWEPz2YzfmqdN3qLUMwOHkvbGWx8qQGvgTH8/ckb7/TzNbjYNdxy613I8HRf2h9fbGLNr778guwcXxEh0GdQBYvzxU2VjqnwMSxAdeCevrrlDW/A0pkzKmC0fqm77bkoKrTB6tbsr3EUTjZ9LFctyFjQoh3hZEJj41AkkCvjbe94L7r1DWytXpEwPPfC83aWp1pVG8AVTXEZbYRGMg1h1SnBqOUCc/HJ3AmyhX5uNc0p/cSf/1qiRQ1P2rsKEQZUJkdlMFbgZ573bvM3O/PKbqgDUehgSQ17LjgcNnfOwlFidkgagR2FoxhdYZA5TKQv8+up03eKSUpEbWNzE7fe8Tqp0XZzZ+R4MYw69+orst100kYayk/dNQKGTdiIheI2llpD75fmsTHfcMeduHzuDJo7NU0QkS2xXvzc6+C0x7OEBov7aq60820xdGBtHGrLa7Cu24PP3jCNe97xbgyaTWxcPa/fsuecAVCR0DGuqti23lvNSpssK2lA0mudYwaaIm26r0HsXJnLB//+vxso6lAmOwT7Jhsttv4uAiJ3+lj7Z1eJRtAzMMVjldFiCK/2npzhrTOjxsEqc+axLwWHfULMKzfu+nU33+HYb1uY8Onb7lSIxpZdro+lwi6cPydIlU6aqVNbHMX10VB+jEQYioQecoSOAfjceNedWDpzFvWdHfMxvADBivt3SUu249wshB13tW6pYkvnkshh2IVrQ/YRVTjIurIEb/7692ix15bPSdjOnLHjLWNnhjDp7G3vrhRahfehWuecGF/d2EVc7DA7ETnIdHzm47+XMDgfSv34PyfmaZF0UhzPf/RmMxa4CfHSronuAj6ZvImdOGelqqPJVAdfO+A1doEWX9CrxMkaqovsZ6f63va6N2Nnh2yMLlbX1rD/4GEcPHgE7caO4mpRfns9XL50CVubm+Kgx3LwOgQ4RlI/5liJTOiHoclPdDVObXP9LTdj+dJlMWnIXo0+M+HHBIEhTvIbuWxxGq6r6NGCeZM+Cz0t2WSwM88USeMt73gPeu021pfOCjc4f+6MLbZ7/+FjKKtHAfFW3LbBDGJVqYo2kB9O5+FmNCaK45hTn/rb31EMUSyzH7j5nYb5+jmY0TpSYZLtCd5InQ7Ey7JSHCMKGL2YixkQbOw07QS/VrAzQ3p1Yg6rJxw2NcnN4vSdr8fm5roQI+5sxuF33/1GtOm5wjQQr7G8dEU7W2fZOu891DMfSrsjcHkXKIVSLqD8W4BJR05cg621DaytXFFPEiFRHFsY9TFnVnVZrloDHYxdZ6cGBbRsjeN3Y347S6SHDO5953vEe1+7fEaLfe7Mq4rVJf5+T/lI1ppAOL11d6TZMc0YZA3RrLxvfKzVa6KRz/7D7wsuDXqNUYqNVmyOWCBj9tCjzkTqG8qdGylOs7k6scZzmrb7DR5VViv8Al8AMUIlheYV6+jBqCbVzn4TVtdW1FNlbXUV3d4Q97zlbei22KbROvJz0VZXVnHl8mVRbCOc0iLpQBpXoe4oUXeF+jaBsNEJ8k2l0Wy38cd/9Ee4++7bsY+JDR8bif969miU4/6KnWoQjFwzcdG3xZJAMbN+JFMQHYnLI4Ove8f7MOh2sXLpqxLKC+fOGiHSVf04UBU5i5G/4AUOfA+F3tg2u5z34BGYtkwj9bl//OPXhF6jvp8uwRZnGjFg1NGXUpqN8yzNSVMxgSNmYZ/ouQZyZuc8ewStE+fNhpla2z1wLVpPJEkGt73uDeKNE3VaW1tDu9XHvfe9HT0S6nqsDrHFXt/YwJWLl1R/TafFMl9GJjTeuFdwqurFgJAwLyNAiAxTb8BnThaBlK44dYahu332tG8cZ2k70M/T8uOVAjnUCX0yJxae2nvjUBrqoQze+Pb3Ydjt4erFl2VzL104PypTskNndzsvhUmKbBvVeFCYAwCIsNds9Wtp0akHPv3HCZvEcbEikRF2wj5odjeAjlGHP8XGpto5SOFkyrCYBiDqFUcbSfKVMTMzoZN6vM5bu+s1xQnWYJZlwjfedieuXFkSAZF9vtge+g1vfosQNMba8fCbW1u4dO78qLOhjd+gzXhZZskmWlThcC69gI4cPOLyjCgsRy0RN36dkn3m8UYyJeLqEOZY9N1FlTfgHrlpDyvCsMZ4pC7TQXvj13Nn97B66ava0ctXlrxvmrFr4npxX9G8YiMyeRKaw9GeCNMsNIOyfqbKE6Q+88n/mZi63T2OgWzQkPgIAeiI6Wxt503HJNruND0tD9CPNLJF9ERJADY6dshaPlscGWrcvGe1+VANOFROdN0Nt+DKlcsiGjJe5K3uuvtNKp9ts10jGZnDIXY2t7C0tKTF3t0NnJTdHSV17tWRHKfxvmynh1Dy93TqZA+9twq/l9fL8NLHGyf0CGuIvqD+jCYg9j9UXYAsdhSym0hWtaQzeP1b3y2zd/XCS3LKrl694nQwW2gzpbsHxIiE4EWAHOO42tZ9RjlFrzVztFBj/cw//BFnWotkDEmLcUOiaHPU6DVtao7F+uqsMmYDxxeetczRRYg2kLHsru0O6lOoNNMXcRC7YlI/gJ1O2613vh6XLp5XcbmOccxkcdfdb7Z+afXaCPAgAHLxwsXRafajSXK0xjQNPK7AAAAgAElEQVSvh0puasxb9zg7doUgVMMR5Pw4SCP8OfBvPytr5MCS+KB22t5wncczSSgClTQCR+z8kXBwsQG84b73Soiunrf4+tKli6MTl0zQrKCB9xcnnKiemxRGH6G2Y6FDsEJj8hoSCP578B8/nNhxjP7gzh6hNx8XEgDiKpHzF2dHMakfGoEDVmd890AD4YrEF+fT4j+2prSzSEjmkzepigqj5cSk5PMl3HT6Nly8eAbNWl0IGXfg9TfdgcpkVa24wtPk37mzFYo4C3bX8x1pcn0TDiHVdnw+nMj4uxweXyA70NVACk+YasxU9zIjDIc8XtdZ2wolY0fSNHT8aAr7tKAdJX2ETeL1971P110+94IW++LF82aHw79RGOzZRvWIsYPkLTHz2ub7Sj2PHEKzmnHagFDSz//TR/ycdPPiVJ3IAckxsA5CmhTufH719GE81CiTNLbIeix3vJi14e6WpvAMWZgIo0BZmYyFDLsxOG32DTedxoWLBDi27RhmAi8Ts7jpphuxvbkyMjU8Punc2bPujVvYGBy0sFcGUY6Lnjkv2oVj7SflTwgxtL9FoY5Br6aZI4YOkmOobd4rMoYyYd7VP7xyhXBuhzWSYYJjN9yJ+YUFLJ99XkJx6dIFT8zsEkkS1xaMDKKq1Ha9JX9Cc4+bFX3v8xtRTurBf/qI5mA8WcBBy5UXROdsEpEIqZbd4Pvp8qPdYS6It0o2BIfgCr/GGV0kPASiEzF2TJCpmzghwHb88eMnFFY98MBnMD8zrf7m7V4a3/QvvxU7G1clkRScdqOJJ554VIsklE/OmSNebqujowHllTnvXZ/EBCBsXxAwKBzWsM6OUQqKFT+vfi2+ix3NlyCrSCKQNkcIzY8wGrOcRO+faioshfmD1+DosWuwfJYdKmpYY6gpLWKJFUszO1FEWDjPzbYiC/V1k7Aa0STmdmS7vcFQYA2pLz34vxJzauyhTUpt0qRu2GBdyQlzZlQ3xPeN8dQIpqhk1h0fE9rd3t4SHnVGcI/WVVnYwlDdcX/aTd6/1ezgwsWLytpkSK0Z9lBvDfHP3vcvtLPpuHCR2IjvySfI8DAVqSOYvSWnhMpNk7xgn6jY/fKmvdWlhWzWuzvUfbBrHdUd/T52EcMqdV3gSSd8U2g+PxMkujSquTZbcuq4rOixDmTKU7iLIea5M1psljqNvH47RNPGz8+Lym3FDPaKGF5++2ixw2FmOXAwSCTsX37of8lmW7Yodl4U5zP+cFBE9un/a+vanuuurvM+siXLsrk4zTMdGAghJc0Y22BjoLSZ5rl56kuf+tfkodP/oy+ZydBppkmAkkkoNrbBKdB2aOMB27JsS7Isy/iiy+l8t73XUdEM2JaOfpe9117Xb31LXYzxtLvTwR4pSR9LgEZeVpvIk5QJtIYnSxJVoAiPCgRAGTpVePBnQizc79H2pJ1+/e32zb11xtpsf3n8qF358ss+WSdIVpLteGFyvWrBs9Gx1QzLEJWYoCejJ1QnF0gDa19LpQHqjKhFJoxQa288TyHYI0pGTcI0abtzi+3Ea6+3m1f+pz14uNlu375pG68hOVhPcdqonJo1wXvt0kGTyQ1zlMRifHEtAgP/+MN3kgrhZuGHkB580V4nVu2D1nSxWD8qy8zI1O53tZh/opU2C0nPO2AFfxbJfKjG/Sc8JkA8prHvc+2Vk2dZDHn0OM342+3alSs97MgIKJ7ylAvLCU6uoJuqMgVQalnjmkZYpU2W5jGO3oyI1GY9RamedAnPKBgBlgQAYrQBrquDMNd2JofaqTNvtLWrVwiWYHrYqNVoGBZhzHmukM5OngfohMUh19f+qCAUT57ZynO/+wWRKnFociFCiJ3qRFYLtyAQwOq8k7LtG8fESlBX4QYt2u6nt5kSywXWwpBxCKrTIAeeOEnQjG1VgmeunX7zr1gQQC8TrgPM981ry4ImdfuVCYBKZgw5hC0WsIGLY3oLLbBKrqlmqZ/NiFW/p+RTAh5SWaP6ugaqmwpsu/7tqlfSpTxYmKh+qJ149S0WQkDTvbGx3hEv40gNkASzcp6AoEepYazVuvMe3XYnawc1HrTJCFdU4406pdfZbbRjYdNAUkpt63Pao0T4kvbMueIGFqpBXYstG2SmJicpFFZgrPAAMOq99FyvvfmXpKcAVQe5UnYet6t/RNVoh/9WGFeRMlrsLB7Xx+YJz8AowA9dVTun7iH37Rx6pgNFjQOmS7gV/BHWA3TiVD8Y3j7u1zeIc7vAMgVth3U92E6++jaZHzfvrfNkax9k4uJYZk1xVX6vqGrlPGBf5LDFXPR7JtV7/sN/0TmK+q07ZueAC+1eLv1dthsnAMNJ1K9tUJ5TlXJsaj6nPJ3Zi4C9Vi+YHERsR8hnnLB3rK/TFOfxe6Cu/s53ScRD4va97bb89dV27x7w5KMql7q2RiaBv7Q8g/8aAVdoOODFiU6kqFyT90LSJynwJPoeJUfOjeiD2uwxO2Wp0Y3yReDRo8x55s2ftDsr19rdzVX2d3HsYuaTs4xc0rV9/Sv2L1UwPKfEQLG6BtoEmzf5+KNfWhvY1ibD5FOZE231L3XI/8+Rfjqgh8R0OhlyukAGD3uM6TScqxVbvSdmhJKnV8HERQeGPSyJJvGhaBfCxbz1wlI7eeo1MiHTmWq7beXqdQLzMk1eWkm7O4odKXJhBomotjnAVKatV+jkUIVpSAyPFMbAjqzNkkJNbE2CeY+TyGQAMjoZuqy5W/DEVeAgwufAQjvz5l+3zdvLbXVtpd0Bu7OdUzw7ng8jq6kNSvGoh4LVfyrIWWpVb3YO8uTiuV8RSox4MN7zrPxLavIL6c5E7hoLMsKA2d9KzMffcy4XQkfaSrSpGqCYe8bOzXrII3VL5KYF6e79x+3tH/+EuC1K8nSPNB5Qgdg2fTYmQCpdXrQ96V6lEkVHHDloCWgBYMz43LGHnPGl9ClOTNS3snWKh5FnZ77dzh7Sy2Ql3tPAG8wCwbVFSARPQA4UNvPlk2fb1vptjuVYX7vFe0k51CaMsgeZQNBDMK19F+p9Cgx97TzhF8//2o19Q8fFfZcS1qnqm20Ok3SI7BcQCcDYJHrDO2itfaiGOzaGuz2ocJbgaSAAsy+pxj1+z2kSXH9j61F78y9+3DZuL8s32ttt6+vrbR1jLayZ9LzJHThvwFh40Fv2iCK8KHZ8sAEsBvnm2EBQhuTa+X719mkryc6gUcbpfcv6wCuI40n8gEGIWOOXT73RtlZvtdXby+3uxpr6203Bid8H71miADwLINQcBxFHLQ0Y2WQntKANuHbOo0w+Pvcr48a1oYq2ZSP6ifZb4nvzC0JW5gTq1CTcGDavxsg4DVBlcsaCWvUm2rusmiD935BUeLOS2O5Cte2duXbi1TNtA6dgD1TVjQD61bVbXaYZYbg2YQnqJ7UKKN5JVJcgBhCsadaxlKgpdBTIQYKZcq4SStKOEh/6AbbjIBzQ9TAZQAT5aYHSlaft+6+cbvfvrLW1G1fbPYApe11cCS4Wh+y0Yj16+jNxvN86BzJ/ZjGgzum/fPrJ+/TGe87XKiRqNb8QFYV226ouqtrdpz1mBCI2T+p1oCFHBDAECCafaUerUiRzmFjh3E7QcB1qr5w63TbXV0lnhc1GVeyOwxY9B3qzTBvhWLg/X46odsZwXyWElFoc5EGs1ZcCDXVdSrbOlxPznjCOZV4lQsgOYZydfADhzxi5USUJRPjD195o32zcabevf9XubK5zs3ELMkfVAbR+NojIE08cJeKOJU+/x7etP01BiAAvXvgNN5ujkKIyi0cH0Bq+hG5UjRpf8H2wAbFR+3PN/Ey3s2Mel2J6PVbCL17fTkw2qsezOiszNeLJ3lw7ceYNOmRomwEVFurda+urM2FXMnYUqHjLAe7vW5nkxvPtekq0L9Ze7DEDoTxoLsBtLt61aB8mobxW1G5GfDLxEu44ok1R25cX/4MfneD1bl77st0hnQgcOCFMD3pONvYmpLYH5kWwHy2SZ0a/WOJ/ijsPixIstNkXzv96mrSe0p0eG8GN1WXYQOAZzIEWIc/dL+i71RM/CgujlDjgsb6uM3bJPwe5mQpVct2Kaw2AJHFKa6+cPkuqRoyMPAjH78GDtrJyvTtMqqPbZsXw+zlzOpMAyp8Jl7KIPZal0+I0qHMC1BzklgFJkNPNwIQDaMdcuzppoImY2vSJls4ZAEccoOdefJk+wvWv/ov1akQ2nLyEWjbsL4afu0NEiS3BrWhanOaWMI5iiEJJ5eO7N/7Jxfd6R8jMD913NfqmZgvwcLoYI6ePiDnzCnbDyRWqcn96tGqB5Md1kmvHpU5zCHPTXMeOyvmF9uLLJ4hU2drc4MlGFm7l5o2OF0tdW0I3SADY2xVOb6NjcjK6SQkg0smLaAVqtzQxWoDU8eFChVU5N3TG+ZTDJg2pJoqOI2tz7cixYxza9tX//ne7ufw1JxbSbNmHSpIIDpmG2TSSDsATUIg6Uqj0j+LQGrZMDBCe8dNL70+hluSAqBdbR9Y+kRMgWNioA0gKOwVdyYEdQsNfWlajgns4ZUjTQFoWtegFzKbIRimRoahN4Q2+xEwoTTO/+FT7/kvfaxvra+yUQBsQ+LWHRrFtdMIoaVTxgkeQMJoYU4+GY1nbd6qmx6IKqKiig/B64z26AHf1OTQaPoj2KHGrylZn+Pt0Z9ouf/FF+5uf/rTduHalXfz9b9t3jj3J+QfJjDG9y5aoxmgGIEgWeTxsjvjBRDhss7b/Yx9BDt+0Tf5w+QPS1ygLlLgl+12a9N0JghoqnAJwimUze2xpG8GUnoefiUZaeCxtYkIi60Z6uqlj25O1vOm6Dv8ywdaFvftb2+21s2fb2q3raqnZ2WnLN67xwYW8CdiwJhZ1/yAyldQaoEQKMdWkCzelb6tv/AgKVE0y5EfCaEfSCy7BVP9XNXFxqOqTra7ebh988G/t5PGX2xLYEiDkOLEGIdAEGlARcGgQrorHkdUDH5oig9Tgtd6mOMPJ5oPkQlalLKCzJQeDxlE8iJ2NLRinI7ZbiyeV5nRy/xMbqhYVLXYqO/SwS3IAzxLkClUZF1D57uScITo725N2/NSr7fbNa4T34HpQ4xAOaJioZIQq1AxpKS7v5yBToQz5VTCkVJuTtJqyqCqQpA5dHUuxUth/KSldLHFKwqoejnC2JksYpcB32d0207JnDXAtlQxi+AZ1jfEW2zucQwZoFt6LnSPBCYDwxxXL6lDOL5joCKFXjZmT1sTi4SEB36WtsXTizxj8bEZ+P6FSTz06hNCNh6qUDRd0SDEkXtQUlS6Q8HeceZMwZdYXBEA/Ovn6W+3m8lVgSLlRt26taHE8CObbMoI5BTFVaEmqz68WWzk2KnP63YkBB4/aYqfPBOYMX0ySlNJjDVsxIE8lysIeGJw8b6TcNZJO0n6D37xGBLTNHALPxXArspklQDO2s0NOuHtb95iKZqOCexnhXzFE+8OnH/Bk9w2HNDlbJVumJvpsthIk+jyrRQnF0ozmPHPQL0mpjkoQZosM1TnrIOhfeDC8PPovgi6hSvToIjiNsIEnz7xF/jEAnHEfqPEsdGL5qPP4EdFYET5ojapOa7go10WFGt6fm6PWpkQuNDJOzECFIudO79ydKGSz8xcFLSFpcQiUANq24zjajqMxs+manKCnjXCR/RkEufb6EYKCkpSQMnKrqYjDeWXZbJbnAhEuD8JeLmdw6oZn07PxgiHLaWHzuGdcRp0GKEBuEoP60BbcwwID6HU9WbugJ9FZwhAE6plqEz+bbz9CL9gaxkI+pucKB024OYdp6QFmbV5NinjAePhpeNMzJKmihnvNDpFGUZSQaESCykDHTfrcLJxId7pogfU93Pewiz5xDHNAcmDI6eJ5nMPZt0BZ02WdsjXSXhJysTS5X85FFDhyqk62Ptpicuniu+JUsXwn5qZnTika5bO8XCQuajwbSu1g+yhbaT0SRKUXVQkUdW0yBjX0iPAbniAFD5wGCRI3jIYKRNdcIWgP+sGfnyAPORiI8LV8Q0R1GuCq6hKEjjPLYJON6aID4znaCZ34bwq7bDcWcjbRkky6kiEJtxiuWhBjfxlaudFR3Z9qicY6UXNgpMbhxe608eCkJ67jzmd5YeL8cfMOmDQXc1p69+hen9pbBQN/R6jKwfCXPv5N3qKoKpXWuHnGnOUEx7mQsyUvOw5RVB3SfLAb8sQ1mTYmS6xC4u5OD1QnZvP1gv4Erhz8pVWNcnQkVOP0QHvm+Re4qWBTwtfNWyukn6A3ySxWAAvyVtP7VHFawZlhpHIydTpxo5iT5E5MQ9VG4CvXe48qm0yiT5WRPemw7KwUtuOBQDEK4LFOAqn4OEVtx9xWf6mPniZ0GcIoAYxGpq2HULDEabWU2LFWpTicmV8KnZhata2m09BbXUZlDJ/FaKI0ApL7k4wOJTwxL3naUxcwjQf5ZJ9u3BEErBpBLCRIQiqGRm2+PfEn323PPvccqSTxhRInrscMAMD729tkG8LG0dPmu3gRDaiP/dVwtREbd3SttRP+LSEbBQ8+OzabuYKR/lVUEpNh6k5DruCvJFNY07Cxw0Go5ARjU+P9x//JhufgAcwoBy5Jd534oZm0T5MLH/0rq1483oVdIBs/c+xl2fqm8WYHNMwktQWcZHCNcpSEpYs5Yo5zkMqW4GhhUapDe5EqOQbtO5QJCyEhSsjWOXTDS2AMIRrjTp89S55OfA+c33BQOILJbI1KWcqRxL2hbSKgSiIp0zcSOXIKs8AAEEbFwjT1EK33sMthGrWV8W69JOq05nAexeeuTXOiaF9KF9eMNoWwc/18GPJs+TlOblXz6XaJj9A10acX3p0KYTEQFUmu0AmxPY8nrGFPQwTojZY4mZOBZtKecnIY6/qUZL7IiKPtnTvMgfCgiiU7rWIB1ZDVssp9ILcDWO9UW13RlN6Nu6tkEEJ2j+zDYPhzxSxISy2iMk4anrrN7s2kN9PrhQWiEBotk/KmzMFgYooDV52umLeo/ZiebDYrab16WMD9xdPucbK/V0NevAM2P/kJYO/w/ELhylzVCCsagDabF+bpHl2JSONFv4v1aFRRdDId4xkpCjyV0psD6Ie/0zFQykhT64o9g4MWPDeegW4ZhrK5vpzSphZ+FDUEPFTv2Cuvnmkr167y5e5uronczYkdqjE3K8ZZVNyMcBJOHGrSek+ke/GFgkpMC+7BU4TnOuAikWktYeOl9r35hjhp2BycOxs/x+3MetnJ1MFBfludKTBP7Et3eKf9MG0XES0DRcRN5vQDHM5RtIr2JC22U8JB4cSBnpz78JeKswtTLz3yvZEZktrTw0hy8AAOLQy3ibSl8Wx42cp88TTCMwTkx4uEFRmqBpkSXR+4NQmF79VhROJbSYQA7rXjp063G1e/5qJt3d8gYgVCxdKsNUV6oiPhym0btEBEKhZdqBipSxHQJ2rgOAr3VGX+p5Aoo3Ajpw68brovpBFrgPdmehmzxgszFKpcMS34LBNYKSfjul1/SqBSWuY77Gl2N67fSXNc3NFUxZiWcXhpsy9+/B6LnWH94xksqqOnMp33jqOGFB4+BqaeWdugGVgKbVBnvt+WOO9aJzfM/iwPTveYhMClU8+G972I4kSHEkNbiJlQEjq0x/bOtJ0+c7bdurHMzQH98vr6Gm12TwyRqQnZJRHEQjUne8dqUkh7Jgca5lknjGKumc6oHDe0KjOGR1vSA00TTn93PO+0HkOYMVtLGyikqPyA0e0Slatr6oTCvMmpVVwvhKlgVPiKiYRgwy/Suks4a7TUEy5WL9xoCEnd7NjQ/FCGXW4lZAWSGbUGT5eDUuz49MDeN8DpTBtwVEzKopmDOUhwR4GCqp+w370+sD2AgIAIEepx8+cW2osv/Vm7uyZ2QHCRX7++zDHInNG5s026aPGaisRWeX45atgcYsvIqCBHM0PQsanyDVwx8nShhGVDaOVgIfqginU+H825+uwBhoP4PLBkAQlkrSEQ2fCUhKN2c/BynWQy8X1om5rBjOfdVbYrez22Z+jFk63TkpvGkajA9rSuYlIffh7JlIqEIKiYEs8RN+8xcWcDVp4Ym4CXxwMDyYm5GrhGkitwsLiAbmLTiXHNuKMolZR55pnnid7cxcjG7Yft9q1bYmBIWLgLFWlqjU5eo9HJQXsQLmQikRAJcBNcIOEkQA+HBSgCwgh4b4bajd5ybW6yWlgLCCiETHkJYMWlIdI8iaQLGvmjqnFtrgNO9UzBTodOZkbTCuTfKIGEZ4BpwM+zrvHQuwBks2OL8+ewJw6H7IFCF3Ni3WGoZn2JamR4h5HIJF6wcHHgEo7lMwT68T/E0wovSKVpcLwkVlkraJP8nDXi6bQdXnq6PX3saRK9ovEdDhoHssGjNEpDmkWxKE6HpuSJ7opwXla0RPADqUtrUJxJOnT22IMQSVO9FlKsSAk3Ewfn5NHj3xZB3UxBCNqyF5ZS6gUEWQPl2CJtxAvuo9hfMXRYDpPLx/tRU1mYoE0gBKHepM934fy7PY5KPJYTJifdRZJCCSkPO2KnP6v6CF1HBCcaItAibeDwvOvvihpT6UyoRhVCNB4i92WSBO2rjx+3g4eOtGf/9Fm2Au3ubLfVdbQEyfFDEoV14eku2RHiiCoxInADrquKuatXCBMJbHQPd6g4IVydiK5kt6zm5YXvtsXDmlVK/8CtuVgH2VRdm3l+1w5U+VPuQRnFsZZsP8JweAsl1gyjkbG+bFAwVGvUuZXNSddJNDQTM0hqZbOTcYlKr3ajH+GGmRaa5BrpRYkwdk1ORkhsArcdUJ44cvlcEgVJFQZUgJ9jQznv2qMaBpOCFTrGP8LxObjQXnjuhba6uiLmgqt/5IJT4OLFp5l9H/BwRssYANE99vCrOvkD3nD9TJtBzWGzpbDQwm+kT0LKqNfkGhA2xbGSI6vWXmUItykETASlrm6wJwWyx+HGFITN2Y2QMHS91h60ivMkPGBffPbvU0gWbqzyn9R0Xjqbig2A5xwg/0gc2GlzrjdqpSaEEuPGS8y196dgByugVGPgSLGjSSRQLbtmjVLn8eMnCDaEqn3n5//UfvjS8/LaCb5YEG2XB7+HmUGU13a+vE9Y8NFtOcq+FE6nP4n/DkOzt5hajuXLAtLs3RwqCPW0rFOyma3dq2k6QqpVu7ukE81mMJo1BIkPWKNSviH7ldw6NWlICwsMmg5aJDXNbPhw3H1me6aN9ihtMREAOQAmijfAQGHUKEAkNSoEptCQ+BPCFQdCp1d4ctko3XMmGgj0Ju01ZleEnf/nd95pZ86cbv/4Dz9rf/93f9sWD8+3xUOLnB8GbxueNuNSsCog/jVlCEMbb3TQKR0IWPq7uA1u8Y0GDL02n7Hi0p0jTZMFO1fpvLoNyZzobAVWQbiXJ5N3p6oHHYjbh2nWDJcCQzPeGeu4uLRkLZsSrBy43vi/73RPLl14b1pZimJ/ZZMVf2MjOLBlH8mNPlP6hVPJ8bG+u3G3PfX0U7LplHrFhUlyKMQTLzgkP6paDs8YDRmTEuHA1VSSVC/1Y87sRBPhw3ZwihLnNz7JiIkftKUlTNgB7xlCL/V7YeKuSAKM9nSbrwo26ekOl5uydez88OmjlvJ7xjbG58m/eZ0219bW1zgkhtqFhRiphK6u4/OUHEc1p3aKmJRK0Yoh3aNHjCggvNG0iumFQuUhKpypk0sX3p9ubm4yoTCcrlrBksUeIL0JHSV41wn6ZcNjmwPzGaBD2ShVYSCRrF512g6hNdNWo8+FL3WEY0m8xF/garFeiGQDxiIjiy3BTCZqfjIhXgsoEKxv4lRQXfPkmesFz/fNN1vMpYcbpfssLKjITmcqQA6CwBpKM6eDJQjcVEa6s1vmqGSjKRRutpDGEeZOTJFpNRoeU54pthtTgZL8GTBuJ19szyM0vBc2OxL57U6ZbiZ77hFNpeEbkqVwJCeieucSfgLj+u8rohWFpuJu5ZI9ycBCoSyXwQ8u0EcYR5Sga89hlBHnj+gLagxOk3LvimnxBRN3//5WO3xoUaB7xPHz8+3QPOLgbaVQd7XoOAAYldSnHIw17/6M1kOFHsKDwEQcjHotItG+ptgj4j/AhHDqMMeD/kkn1TPmb6YWoG5PxuNYN8dPoAUPlmCsDZ5JPDShCoFJo4N2+ZPf9s3GpmdTojKrg5bNrp57PNrYOth2Zc6GdqAtBidocN8Zv5S5GS44xGEj1bJDF9zTfaSdB1Q+geJ7OVomk7U9xKhGxZdqm03SvWYI8bzppWIee6IRj/MW3m67HSaBxTDpzhyO8RwqicYBlUPmvHRYD0ImaEh2h3V11gph/ygwKI6Y3A4nPp8VocCgueRmylPrzA7adIV9cFjjNPJk/8fl302JPCzzr5SEGHTGRajlWboPORs9q/5lnxlzLqonKaceJy1pPZ40Oyg1BOLfozatQUgQU8hsc7+Mn8pmRwPd37rfjhw9qkEpHuGgbNkA62Xj6Yi6GY+x+67CIWwe1b5LuECSJgYGGPLOnY127Nix/2f6IgjQz2n4i9qWdhnVO4aedvwQdiE7FzPFOFzODu8xYGI2qRMBMzmG8cA8w9T8Lip5iXhkFg4wvp98eumDGXxCbHNOeAXwRwhy2hmse2J8atjZCHnYvU6mGZmeZ8Eih73zOEP99+yJ8h7FAcLCQ+UlYpAfIMHqwuZ5liNe1/35Lv4c1X3meblJT8+g08HMFNbYyBPlx3MPwZ8hCIFSJSunRFBoJvX5/VqxC2k89jIlKbZ1HAZBmxSDay112jXgHZ+7t7nJwg5VPFuD9sQV68YFnHx8v5c6ocbjIWsBRzEdL5qXIpDPbSfDSYqNnG2pqfYDf8c1qhbQQBi03oxMnDzYQTyjQHH4CBRyjDGiFtImI5SS1BvAaK4xLBJ6v2BSxvuMal7i+TwTFjNdILDdMDlhJkz7boQ6WMpJKI8AAAdhSURBVHeFTPM9/Rqn7SGm2TLZokWOZ87nJ3wJFTxtWl2TCMY4SHD8nO9wf7g6QhVbU70/gokKBbj8VZk1NxaWfAk1xOXLv5/SPhtaEw6x2G+l8gZTQiQvdrtWYvAgyYpF3UeAcpry0hEYwXoH9kzJj9mxilGfta0X8SbOrainFL5xRkhaVL0IQbf0Re8/l6DqkMlOjAVPn5g1aY+5NQmIGss4M5qJEPO5g0MaT8UTrB9ULNYFEUzleckzVXufE571iTnVeqpfLHYYzI442VwXLazv6VYuv2tMwOSzzz7iZsvDEyYq3mtuPLJiY6pMNjvqvnrrWqJxklIQiGpXCJbWnrGxuSayXimPytFTokYxcwowOfXwgBH/Aq9u4rze751JQGFuHAmfoDxiampdOUmdYQORFxdiFT8TJaZBfGFWNudKjbBy7RD+5tBwhBRNgRJSWQtBqPT90cwY7nIsqPP5ps0A4RBKuHpOTQfsozhKQ2OHlGGz8eHqqWbzUz8epzykqFC5QY1kY7Upo+gxWoaG/R/9xFGvtQ5bncR45ji5meKjk5ci/igYxPGSWgRXqVOdTswM4cvfIoiBGAffpsORcIr3Mxl+/02364hFQdGLBFuqM4DGrBlMFd5V5rACE3WvmkmMd5/3UM1cdfZ68GifbVblAMuRC0NEogL+jgs+9Ds+//xc51SpH0p5MKiObE6kKDndqp5rPbyq8bHE+lskOLadoUahg8qmj2sPxCfGIIhZUClQePxaCBPjwvbbYQmNNq6TGrJSkE7d+lQmWRLnbzhW0tUiBxi5+pz4qn6x2XHWlMMPBNgJmd4TDm4ZIV5qwTo2/969LQpGZ2xy/h73TBkzZgIags7XnCpd1T/oG02NZ8QrNjtSk1NWN50pOvdJMzXKAWUhtk0hAY1pGBAumqmqKbJww2kbZdMqEJHq2PiYAZkQJVeGV6xTgRQu0SX2/BGC4GVUsx5hTH+GjGvEe6BZgfPHFCb2cMvJnzwP/qQ69vgFePO5djZoqOtBWJDTCUEJiie16W9zziJAua+c2j2GeEAE6T2Vas7BgBMatNDsgTKYz45sYvfJF1+cFw9anddRSlYjoaHm+AhGbJaVeMc/V6ejhh9V6rT4aQ0a6jhCNpw6lDrdb+wifjYuzxsBVSZPSQdWoAwqYJxpZ4mkcalU5cSYKuvBw4fUEuRutIOVEI4LzchE+Paoea/GjI8Th2q/TzLUveJkkcQP9RxBzmZn8/P9CBQg1keOLLloFKbkUaHTvjjTZh5Xric88//8XDZbLrw+GDWkgsUgcmNhxMWOvExV9yqciAqK0GSX2YT+UP6bed2OIEHixm1GrhvHo8c1hkerNtZasKnhHTZDi2xwIBGv0DI6BQinDh9eGsCA7n8Hj65wCM+IpEo2O2iQnETew5oDahYLOBoAM21wIGarxqwaLhmxmouoMbjWAKp+ND5mPaJpIgSgBHvyyaOMtSHJ/YAZCxw7zh1WnA0vT433mT2ZBIqw0XoBVprc+hNtkOZb/Vt56H5Dj3msKoZ22JmsEepI3qr5iGceCR8/F2xoVqWbu6yGHkUooRJRi0fOLoBJBR8WPlflWBErPK54huQa8g7yA8yYmNGI1hJxxMhs6CRLTqScqoH/jg+E90h0UgWY4bCLRtV5zufzp1S6+VFNeAAPPbTfSSbxmZFBq55xJEc4LcGH5GVrI0EAQ8fEpzbSmbId1zDcV2bQtVfWwQL5d+gngCiJk7V/w7UnmQ44xk50zeLwUvH0MDNYhEMkiEOodJA0mouHl8hJokze6GGTf+DZIrPGr2cBq9kQkFBCzejezmWEPJue39H1k6cfEYUEwKEVhxBopHUEJEIg1a4GSp1wMSly0KyjBX7fh4BTfQEgdXMh9hICMJMujWRp4VVPjuufF+nqPjXYzgIgz5WntcTY+G74TmP0qTWcqWMt24akdk7GpkvCR9twTnwWJPY/mw2nJeqf82bNTMgcOMuhYBnU6GcszsEF0UzVzc6192ukaBeZORMRWJtFSCMEw2fQy+XfEhTXsn0N2nN7/DtZF/8shy+Ck/tqr9CSrGIINS8STNCsPjwo+vJQhEwAanxspLzrYMJif+Nc4PuCz6rmTKkMrpr5ZJUsuTlWCTOJd6vW1H5xX5QZM1YqKjtOVcITLeAgxgkvSxy54cmbiNbsDTwnlPgQ9nlSoPlX8axy2NCgGF6xkf2iBpvF8/YTHRUPXtCcQDx3nLrYeTbulRFMSHAwDGQXrUqwOKXEoO3stKWjRzsQQSHfWMH8HUxK7D1zFm/A39y9KenyaGlV3Kmlocbria6OQiS7OkuxPbKD8F71QJ1+0r9E25yGP6u8uvFU/24zDYlrdVjiE6g47+S+a+PDdAxgdU5U7CliWXB2Yqgc4LoLwHujros6d6V4dmGB7feO1SNssPOY5Y2vsXnjpPJeU+H3EhYpATL4YhB/R4j7oeImSVvBK4eNX1wQ5psACg+hjQboPlCiJm72nAbYl0oe7TS+7/73fRjI9n85OQ8T7wFtAwAAAABJRU5ErkJggg=="/>
+        <xdr:cNvPr id="15" name="AutoShape 14" descr="data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAHsAAACkCAYAAAC3r1GFAAAgAElEQVR4Xmy9B5Sl2VUe+t0c6t7KVZ3TdPfM9ISePIqDRhqhZAn8DMu8hXnPmGXAawHCZDDmwUMYk0GABcY2wQSBSBaSQBKDNJpRGk3OQTOdu7q6ctXN8X/r+/bet+7o+fbqVene/z//Ofvs8O1v75P6ylfuTwaDATKZHDKZDIbDIdLpNHK5HJIkQSqVQqFQ0Fe++Du+n7/j116vh1KppM91u11kUmn0ul1ks1lUqlV0Ox19bjAcYjgcAAkwTPi9XYfXKxaLun7cm+/n/XuDvq7fbbfR6/X1Pl4jneZYEiCd1ec5Xv7ni9eIMfIavC7vw1fcg99zrNlMBvVaDYP+ABOVCjqdDiYnJ7G+vo7+cICpqSmUy2Vdj/95bSRpNJoN/Y3XHQx6+prLZFGv11CpVHQvpNN6P+eB9+X99Cz+lXPG8fErr93v9/X+mAP+rt1u6/7xe36en4n38JHHfx4MbL1qtZq+JgO7ZjabQbFYQurRRz+TJACyvtgcDC/A/5zAmKj4ykXW4g046fZ3CklMLNcAyVDvyWSymkDekO/JZCgIPc46uFx68H6fP6JSqaLZbCCTztjkcuFgg09RQAYDDJNE10mlbHIyubx+jjHwPrwff8eJiYnm2PL5/GjSY3K5yFxwjovCx89SkPj+drercU9MTIwm2+YgrbEUikXdo9Np6bq9Dt8/0PizuSz6w+FIiDlPMU6TBKDVauna/Bs/z+cZF8zYWHr+VErvp4A1Gg1sbW3pd5VK2TadhDBBqWRj5TU5tkzKNif/a30eeeSzCW9EqaBUhzRmMiaNsWt5gZAwDoSf4QXGX3wgTjDfpwE2GppkLn08kIQ+AbLSHKYN4sFarbYmm/fkq8MBZzJoN1vo8/tsVg+RzmYwMzOja8YYOAl8qPHdHRPJa8Ru5vslKJkMEkp9xrQDBW44sPFo0pEaCXOz0USn28G+ffuktXRPLnCvp89QSMoTpp14T16f8xC7lb/jz3x/aAj+HEKgsQ+GWshWp439+/ePtGyMnfcZ9Hsab284sE3A3ZskyOZMI+dzuxsxFlnP0uuaUHGxbQdkkMvGg6eQplhwx2ezI9XDwYeKp3qhpPPv8Qq1rxtQLfUHSHH3+04P6YWEwXYIP8Ndwr/x//b2ttTOxEQF2byZEk5Es9mUFOt+aVPNMRG8X71eH/0cE8txUfXHK8yGFjpJkKdK5GK128hkM0hzTLwfhaBQ1L34GalvQIuhuTIjos/SJHXaHZTKBY2fgspdSIEYN4tUrRT8MIn8Wwidmb8U2u0OUukU8oXCyByFidI4+n3kc3kMYLs1TClNCe/ZbpugmrkbjjZNMZ8zIX7mmYcT7hqqU74K+bzZwIxJTbw4UP6ev6OEUgVJsoecexOOUCGyYbk8qKz5no3NdQ2CExFmQjug29X1ymWqnwES3xm0vnpwV/cxCqp1jqPX7vBxkc3nJQSctGq1OhrruI2L3c3J54Rwgig81CBSdy5wOZoPJBgkplI5YVxYCdtwiKYvYJg3PsfOzo7uqUV0/6DdbWsecrmChIjCzvmlLdd8pmyhzBylpJK5cfjM3ADtTlv+QzzDxsbGSHiq5Qn9jf7EuGngfIdW4XxwLkJ1x9+kbb/ylQeSMp0E38X8pe1YU9vhjPHBeSHZJ19sk54JORJUg8WiSbfZNu6+oSai26V6tuuFitNuGZrTw50sByudNtua0KY1sb21je2dHZSKRRw6dAirG+taBNpH2ihKeKjDuG44llxYTmjsjBi33i/NQ7tb0PWnJie1O+kzFMsVrK+tI1/IY35+fuRvxFyMa69mo4Ecn6/T0Rj17IlNfKfTs53X72sjcY6pwQqFnNQ+BWVlZUXjp/ks5vJaAy4kf8c55e/54nzKbGbMNNCMhXaKv8VGDBPKcfLznA9qPdnsxx57KOGH292+VEkpbxKdSnEf8UY2aDpwox3mNjkmOLzyojsLcsiovodDPSQH1u31sLW5qZv2B2aLudgUECrJGKQW39XpoD+UWjOv1zx/Si2FiLuF+jSdzqDb77k3PpQnigGwuGcR9Tq95kk5W/Ja+wOZjjTv7d5uJksHic5kHu1WC8ikJQx93y0lqdTE7pGixkvrs7LJYcYonM0mVldXUCwUtfuSlO14037uZfNGqZTsLn0AzpG0B4Bex7QOhY8CxMXms/Kz1CKT1arMDl+r6+t6Xr4nbDMFM3yEiFBC8MOZTj355BcTqhpkslJFGdDB4ETa0vZ6HQ2aaom2iu/lhHJgfJBQY1IX3M30SD2Ei5Aq7DE93xAgqTEP7ai+5Xi5d08JplXs9xP5EXxY7cApk9R+zx2gQR/JMNEC8R5JYiGWpCexHVEsFTHw8IxmI5fNabHtfnwiap8ChoNEO3B9Y10LMj83p5+7rbZMVofOkdtwOUU+rjATw56ZQfkrFNi8LUy300V/0Nd9ad/Hwz9+Nmx4q1GX2s8Vzcni83CMVPGcf96v1WhKC4bDG+8L7ztsdcyjaVWLKjS2Z198IqFNkgT1uihkcpK8YWKhQKgLTjofIn7mLih76KAwhwvsNl5T6HFpSLWkjB6jS608U9nOtNSSpLvXe02IRBulsML/ZuaFXrTZPE6IHoKeJr33rsX0nFhei3aWO4LPxWeKUIy7k2q81W5pJ4a3TO3DBdGOTZuqDDVqiwp0JVR2fwvV0nouhYa01VzU4RCFcmm0q/nMNCvhryhUpUD7HAlTGPakbrm4IQAjjZBOj6KWcDLNL8iNsIoILWOueL/Qlvydnv2p5x4RqFIulc1uwzzbcqkgCTdny8IVOSeuiqhCQqJ4oXBcQm3JexwMMOngQ3jo3FUCWuiM0V9JpxRiUUVxYSOc4PWnJyfNi4Q5TXpQJCjkC/LaeX8+JD1pxrdcKKp4TmIsFEO8drulxZVJoK2mk0YB6nYNtODOd+eQO1iefio9MkXUAAp5ej20uh19nhM5HkoVsjkJlRwlmqGUCW84TvGZiGBoMrtde26Fn7Is5vxyTOHAUaD47KGyuXBzc3OvCWUjnAuVH+qb742/6XpPP/eogkw5LcMBCrk8mrU6si6hqbQF5IWCxb5STZykUsnCKk4Mna9koAGN7ARBAvfeIzzjoLk4dPT4PqpIDmK7XhvFvfzM7MwMWu32KKzLc6L7nDhDybiLqRppTkpFQ6K0A4e07ebwaVe4g8j7Npst/Z0mioJRqVb0lYLNC3KHc2KlGt1eT9BLdmSO9+ecMIwUltDrax6klRJaDQN6KMC8Hk0HJYoCxleYNOogaaFOR5+nNy6zZ2/D/PzsSKOG4JvDa6/xWJ6fD78gMA5uAqGh6YzubethplWLzZ2hsCABOq02qpWKSSehR/q83ClpAwG4GNyx3DGx66QmcqZqAjyhMNTq9dd486PY1uFBugU0B4VSUXZ0HC0at4+h8kIoQ7VucXfT4XEAQ0JZNGiXoZs8dtdMXCyzm4kBNPTUM1TBpgWIehEmrUwY3KmFpOYo5PUzr5dn3I+UaRIHXei48aXQldfu9qShKFjTMzOjiGZkN31M1BS8PwEbLUqhgEa9gYmKhad8hWoObcnn5FgVkfR6Ei5uHL4/5t6wCEMWBU7Rdxmak5h66tnHkoBAOVmUODpOmXQKDC3MVqX1gFT18pZztDe2k/h3gg0UgMCF+X6qND68QhXChfLOzRSYM2UOoL6nL0CwJLHYnrY2Yn/6CozZOdGESTWRdK40Jj68LZjtPBfIlMW2HCvtOHetoNax8E82t0sVaVJvCF0GRPEYslBI+FwMnbhr+ZwUBMW57plzgTkHfF5BpA558rliXqYqVY2NWobCymcNDcdn1Wd890tTMqZniOvQzfT0tASJG5DzEoJuzrAJGsdvttxQtRBwrolpV4tkUi+8/IwjaLsgCgdEEF0OBBfL1Qe9VvNg9QtHwMzrJfTJRaEKlQfoi0nEZ2NzwxElG8y41MbgLTGRlwoM3Jzf2QLaAyREy2lfAallhm2cVH7WJm4gf0A+RD6vhSKerJ3q3jd3KLUBF1DXSlnSRzsjbQ6p7bAKehJYe1ZeK9RqxNpyHtMGJnEX8sXvhTJms2hw0YQZ0GegYAwVj4dQclEnpyYtOeTTyvFwiiLMpRAqWnL7G5uEfku9sTNyOu3vKdn78MCZhyBIQ8xEavyZF59OtIiZFPIZokwNvbndaqBcKGEw6KPoWLW8c0mK2Sg+kOBFd3CUpZmYGDkFFBpqCmZcwqYp5u6YrZH5cODGMjp5CY2841xOmoVj4TWofQK14wSGdqA24WfDWYoIIkIcU30ptDud0b1kagbEx7N6BoEghCzTad2Ln+H9+BniCwZYDLBTq7lQM2IxRDGik1TWsk0Ubl6bfoZ2snvcMZ4AP8zh7KM6NWXJIvoXBT4/zUxfmkJ+1MCwBjqTvP7U9PTImTREzoQtwmD+bmS6uhQUcxilgV4++5KEiCBARmrUEBxmcxT0p2jPbUcRXOC2swU39IuCwt9x0gjtlcplhWHh2PDGdQL8zaYGPlGZ0OcD2aIzxJ/lpPCaA3P0qpOTI7+B15eEc9CDvsKi8GojpjR1Y1omJpYIFe0bNUCn05ZfEF5xqG6ZBU9cUBtQi0i1e+aI9k8qME3YNJGGKJWKSIa2kLy/wKVCVosRjlK/w4wefYMsCDYF3Mz3M2oggra1tY2Oe/Czs7MygxGXB6bPZxF27iqeP0sQ220JFneurunp1LDdYSIVy1PLyWY//1TCC+RyWYM23bGhyrTQimogh/Qw0c7iwwp6c4mykMrsnh6eNtRVeG1nR6B+2DA+CCVND5LQqelJYmWvlRk1eJYf53hGgMWQKnoXiTJNZHlzLmAAGgrhaNv1ecPCeT8JL737HLFuy3QxxuZX/p2LaGAPowWOlwtroVOnZ37G0L3xiCzCpvO5OW+0n51O10wLkbY0Q7WugKq+A1S6n4dk/IZhF6OOgKQjvOQut8RMSiqcY+dzxqbgnEYoK83nDhqvR/vOr1wzCgId5Ugppx596pEk0Cthub2+FpXOkGDPrCUMUkyMM1HiMabCINlXUyN0lCSBvnDcoRQMOkemWgwjpvetzJDwdMavGUkdFzqIArHLLRwkNErEzAAOLgr/zpBJpoC73L3rVqcjIeHc8p7joQntI69BoRHSlBhAxPHH/ahOI1mTTpl2IronGzow7TaO7UcsbOrUEibUVFqklAMy/S7o4kWem8/ATcB5irCJX/lZjpfzwu8j8rFM3FDzzh0aYaG0WJ+hZl/+CZ+DIhs+Q2g5aVHOMX2OrzzxsBabEs3kAzOblvUpyIYw7JG7z90c6kJwqKl0hWeesjTPkHivQYMCMnyyeE3loxXSEK60XTk+6GBtmP9HreK5Y4kZUKvtaLG1kxxk4b1MJXeVaJAQuoaIxRMY4lkrM0kWr3Lx5StwEvs9MK6mA0cVST/DQk8TLu2uMUcp1HVMrrJ2SSJvXlEKIxJh8gyxnGDhmTV+Vo6TmxXZW0LGLoiBuMnhYx6AGEOwcTx219iYMWQmMaITwsaDwUhg+RwCv3zTpB5+/MsiL5hX20POSQv5vDkuXGzFa2RtkHLjoRQnmw+hz7ojQlvHvSc141SkwMM5cE4Y6UWUQEocU5sUsJBCxdF8KAdPtOMUqlhYRc1gnrQtgMXLWak8MyW0nwNPF+6SLwK8oE2kAIQTQ01C28nPa/cS5iyUNEFcAD53eODhcYd9DHAj7DavG3FxhEImtDaO8C3CxDUaNWmY0A5M1hAj4M90TCm4XGgKJ0OucAYDIg0oVQAPYWeaNUfslDhyUItaMfyY1GNPP+pMFYt9mSDnhxrNuhaYzgWlqpwv6uE5iAjutbPH+Gjc7bSLyiyNATDSAo6XCzcfZc2C/ODok1N0LMzi5Nv1OB6OY2enprw3BaxQKJoal49AEoGBJYwciGLxPZxkqr+AGyNRMA7YRMxLdWjYQErXpSaIxYisGxcu8PtwgGKxKbTB6qGm0AJ4WBhUKQoRx8+IhQIsP4SIH59xLEbnNRk2hRMs6Nk1JXludHjDBNIp5Pt4T3EISH4grE2giBh8Pi9TKij3iWceSyg5TGVyMFnu7I57fz2qtJYgSdocTly+UEK5zLQl1bqF/nzI0A6GsBm5kDtcUF/CHWuYeAAInHCCFoa42a6MGNESFvQwzQwo/CAE6ULEh+N/20H8m/JAcro0CQRcGC83GqOxxU4Nr5XPKgH0JBCvx8WlL6A42Yl9kXjg89GX4c+2aJaIiMWmg8YF4hgopAzBNzc3R7loOYtyuIxXJ6zdSYYUNGooJm20OMp7M09uiKRsuzuIyk0QtMmksbOzbSEI4+uJsogYEcJFXB+OM7GD1Jce/aJsNrHtGj88HEjd5tMJup22EvrJYIB8sYRSqYzSxASq1UmUJ6Y8xKKDYyqf6pA340LRVlG1cuI6XebELbnP0IYTJKTO0Z7AfkfeKBGxXneESAkJC9za0TeaAJoMjr3bY5zqSBi/IoASU9nKjrmpUa7aKVAUXu7+yJ5xYiIk5ELyvzYA05m9rjhoy8vLyGWY5m3ImYpEBdOvBw7st3yBzBnnxeJ2vm9udlZ+TrNFUqUJI22tOZ4MpxjimQOby+cUVnEHVzwCoqqTQJaK0mB8z6WLF0zbFkpm5sjedSda8+Kw68hmf/mxLyX8ZaO+g067jmGvIyZIPmcTORx0iOojRQaGXPoicoUiKlML8gRJdqA0kiJEOHUwNFQqGCfaCV1yy7bk/Fy4cAGLiwvYs2ePecEOH9KeinjgryAdctdzh8euNrtkSX9OEAkKVOMUDl6P/zlew9oTQY8kSWSFtqVQKhSxtramu3CMAUhEJDCeOQo1zK9rq1c02advuwOf/Ohf49a73iCHs9M2XDoyf+F/MKdgmT9T54pcHCfgV+IOnLdxti43bbtlISIXmxrXHEFuImozmxyxiJIEa2uGIzBvwfmi3S+VLWFFTaJMpUgWBqumHvzS5xLyoNu1bQx6bXQb22g2ami36yCLI5fLmFpk4l057RQq1UkgW/IwKytUh7TeoiQsh3K5guGgj1azhYcffhhveet9MgecUE4+NYFiWIVK3EGkPNmDmUNkHjOFicTDRsPIhJxsqubAyvk3OljdbkdmCJ6WLOSpRSioxptmOElSgBZ0OJR65cQyAgmTwPtywng92UDPpIWD1WvXsLm5gTe+5W34o9/7EN7zDd+MhESO7Z0RHsAJDQHu9Q13N66bRR1yNDNmvgwhsx1Oc2eQr+EMNJvUKPSsFW45Pp9JG75BU8DfUROb+bHsXIZhpwSKiaqszKbRr90UfvTjf5Vk0n3UNtfQbzfQbTN+LYgmw1evb+nMtHO4h4yrBZ4QB88jTbJDvojiRAXF4gRKpYoGJL5VviDItdHpeVrTmBOBo9PmcMEIhHCSRdFxZC5if+4+Tg7NQLvbcWpSRfE3QyXa2Ga9qc9ZmJdCtcpkRV8U2vg9J4PcdArG1tamcHZOEjNh/EwQB8JciF3rW4mfbTS2UdvewA03344/+59/gG/51n+jzygJJC/egB7aawpKs1l/zZgsvcp8g6U9RcaUo2lzIoFwX4S7lbtaCaLQViOMwVk5bhKEySeGFWTyTEUXTJspbBsI8qVzq4TLX/zZf0u2tlfRqW9idqqCen1Hu6TXG2gnKF/NZEQkDpwJkmT5YMwDTyBfKiNXKCObLSCdLSKTy6BanRKVaXpyGps7dUPcFN7Q4zfHy0APc3I4mIhZd4n+fVQqEyIMcFE2tjZx9uxZLC0tKQ/Mscnm0oZlcyjm8zh27BiOHz+O6ekZdFpG/Y3EA2Nnzjb9kJ3ajpH0U4aARXjEcZjGsR3HCadz1GzsYGdzDdfdeCv++i/+DN/2r79LGiLoxeMevj1P1xiwYv0MtYvDJ1EWjQkPX/TAsoMsEk5faDja+OAO0P5qw4CgEfPvpEQXjXiS92oRYhTOy6P/QPuukPnDf/rBBANOWBubqysoTzhJYWjlJ5Q8euIcSHjc4chIEDI5qZpMtoBMlra7gHxxQna9Wp3GxOQCElJkCcP6i+GdqjGodpBCd2ATzAdReU82JwDlxZdewksvvYS1jTX9vecxcuzWcOzGVfHoHtz5JUYPBczPzOL06dO44/Y7BOoEZYcLFHbbgKTirsOWSrQjDB2DdnV9Yw2HT1yPhz57P97xvm82E0LOuUyMOUfhW9Cho8Mlm8xQivj5iPtmi8fn5e/DmVVenqZnQAEzDrrSlA6bCqyhqePadNoCkoQRgMCNcpNmNpywqSSVo2rSJb/xKz+eFLLMTfeRY/oysbonVmGYnbGgPC5CO0Q3n1IXjpI8cd0ASOdyUunZXBmV6iwW9h7FEAa+iKtFe0ywwGNvARwYKmy5cPkSnnnmGZw5c0YL0uoZm4NaRQ/ioVKABLHYoeqCIBDhEgkVfHCKFBedCRSmGMnEvOmmm6QFIg7ns0Y+X0BFwsXxWjKyaTZWsbp0Ea+756347D9+Cm++712iRtEfMNNjfLjIm9PTjjy9tJrnlhU1EATSHBAM4WLtEhW5Uw1MIQ/Acp00WSJe+m4NoCSfI9RMoqcnnpwzyKRPVI44XGj3+LX//P0JbVKxVECKnGXmdJkA8cUhmCV97xmeqMXiLjCuuZH7hCwxFOoPMTk5jUw6j/LUDKbnDmFyZlG5XQoMUbrI1jIuZCjz4osv4oXnn8dOoy5HLZIe8mYdirUFNI6a0Qu5YUzqRy/BmYwc7DchFBa3GzrHF8fBsIg7l/7I1NQ0bjx1CqdvuUVJlYjh47r83M72GlYvncPb3/3PcP+n78edb7pXBX6tesMWeWglReZMmXOpHcl/TvlSalh+gKlxIYb8zMDoTBEi8omocZjgiKcbkFYfxZBD80+4QfVMJC24phDsyhwFMQg3vYFmpn7xA9+TCIhPBihmWQJEN9/LdrSjzdBzNxIrV/VleIeUfDkkeaRdBXECaZyZCJia24NuUsSpW+6SNy4MmA816GNlZRVffvQrePXVV9Go1XVN2mYLxQzgtwW1laMW4WLzRS1iEmsPPVLd/n6S+cY/GzYw3isChvLmNE/GvEwPWVxYwVS1iltuuQWnTp0aZfc4ofXaOlYvnsPdb/46vPLyqzh2/U2y2TQtlrbkeI3kwBeflTl5YeacI3rVjoFHrK9lF2c9IyxD8XmAJq6OhRYWC2hRZauuwoTF5sTSzj4tUtkULoOxeyq62N3ZKaR+6QPflyhWywJDJh6YRRrS1hhFKQj7uyGRTbAyQp7jNpaG2fRR2pDFe4UK0vkqbr37rQIWRLYf9PHZBx/AU089iWa9MWJNWrxrFZ0Kl9xWxWLbw9kuEanPvW89rDMzYzEJqkilxxZ3Idjd2TZ2qVenKvNnyzkbIsg5IaBx04034fbbb8fO6hWsLl3AqZtvQa5YRaFcVdIj8TqrkTlIGS1bfgSdUa6E72gOWz7JWHgU8KuhjtSNxgW0/IFlBM2AkZJlSBsdM1HFXJOEuFui1lBN2/l0DFmk6MLxyz/3/oQDK5XzSDn91x6YWbCWFps7ke+PhAM/Ssg0dlxUUHCHh0dN9d5Psjh7cQXf9h3fJ/L9o08/g8cefwxXl68YgDJWSx1o2jh8GQscO9cEjjvbfIRQ7UNpZ+On0QSxIsScGtMMAlrGXiEUIUghWJaZM3iSU6a8fS6DifIEKqUK9i/M4NSNN+PW2+8UM1aOnlivu4wUwqaMDOhAEZMWS5Z2WaQI2wzyNZzRqw3j5BAurmWwGN6akFD70L5TG3EjjFBGpmhJn/Y5ZMREDSyOn7Sikys4D4Fs/uSP/9ukpKJwMk4oUgPk6FJ5WQztIyU0EhvipzG0cIaJr7iQLKnYtNVqK8eayeHVy1t45zf+n/jkpz+F8+cuaCe3O1TpVpyuHUYO1oi44EkT7TjPJXsFRnjd8uG1K6nGBhh4sZyx12yhtcjK8VqJsNlHI7jF38eFaFybjAtHwKb58gQI1jA+J4tmfmYex6+5BtccPmDeL3qkfouuJIFNzLHV7vTiwVjgKPYzgQzv2ahFgmY7lsAJuJNzTY89dr9COdaBZ4NGxXsa8ZGOXEC8xrBJI0XYlvyBX//Vn0zajQYmq+Sb9QxtoipKvG56wNJQBu4GBngkotooedJEZ+QtkqFhD6b0Jx2GXBk7/RKefv5ZrG1uIDUw4iCxbNpk2maFcz7rsYBhm2PhQtWG6chI4o0LpyyYCmK4iJT0XY41d7+WX3YuhVTGhGfcnsf3sdvHfYBIJ3Lxc1TtBZL3c0bu4KISfi2X5eFP5LK47fQNmJmwShBqiBFU6hUZdLgshbtrPhgDBz4fwEqMyWrJrALGVLz5TwRvbOGNI9DvGRaiOfDUcrBc+DMxc23WD/3mB5LN7XVMVSYsC6UkeQqH9h/Bvn17MDU1o52aLVWMJeElran00PK+nabiPe5WOhgE8pP+EINCFc+/chYvv/yyUpO0J60mHTDzsBV6yNu23Rn2OB6Uv1eO2RhyI0+aP4loPyq8J2Y8MJanY+KBfAnpc7LguJMW34f61jXdU9+140b0I0TJF/EDZIj/M+WbR67AxFBJDpbsvfyeDMrFKrKpIfbNVnDztddKEzDC6QtYoa9jzQqIVyszSIoVee6OM3Ac0nhjPooVRXhRorho1q4EKdvhUTYdqePYHBIW2vVg5Xz6H/4k6XaZ5aIt6WN1dVWkAuKvlCLaHbryzIpJUl18xIPOpOTFmlonamRgQJLL4eJmGy+9+KKcLg6e3mGzaYjPSK0ZlVrvsV1kYU+kN7ngI+ryWDWE/C7PiZvN4mJzZB5aOcGBJsfE3VKioSliYcMsjNvzEDZG/0aiMEdIi6SEQxHFUkVZQC4UVaS0U8YBGAqiV8jksmkUc1nMVSq45aaTgobTXpJLZyvoybLPo1IdY+2qqsRLltR1watCtEPdQeYGi9DLtoQ5hTJhgp4jXrcwL/UXf/RLSqdQCsx+GrbLeqSwlLcAACAASURBVGVKEFWFpQB366t5MzpYVD9cSEuRplApl5CvLqJXrOCVl7+K7Z1tT/dZxobCwCR/qGsuWDgY8RASHKFK9PAt8xYPZ7nrFLIeUlAABfprt7CyMoMBQ5mITp1HF5LOz47b43FPPDJc4dD1B8zpm2PFCSSOzs8TFqbJylcqUum5gvVqSWjC+kaUVIHgwHqqsFxI8zrsygGeLGXx7ne8HSxl5D1VvizqtFWrBpUrtJIxTswkBMxqxY6SeOcAmh/i0qy/8dmiPs1dFqR+4xd+ILHuOlbiQlBBXQdy5FSToGDeLKmzQqpUOG/0YpHbvc0EXaFBfhKl/dfiqYc/j3q7hW6LjpgJCz9HDjZBei6MFtE5zrHrAgkL7jYHH4BNCIF2WYQXopsx+LTnlKOUIZ7kxQgeesX1YyG/NpwLTRM73cIWCwNDy1CdcxMYPFxEkiNzp4wkYzufQsD38FqCdj3lmvI0roiVFM52C1tXL+H2G6/DO9/5Ts/W2diJZ/Mlb97JFRKUsZKrCKtIkmDVjsHYHoV4XxjLqRv3PIAcRQS/9cs/rG1n5D9ic27nvPoiiuRMzbgO99KfiANbrR0MhxnsP/12/N3f/SUyDnZQOxiNyJiTzDoZB4w/m80Sb83VdYRtob7DBsm++w4Zt62pUH9qCUVfg8O3/HHs4PAFIqQLJ2/cRxjH2GMMDKG0WxyNE1qo3LLVUTHTx8RPJl9Chg4se9Kwhj2VQb1hiR9OGGu4FF4hjXTSQ7NeR7u2iU5tE//ym78JJ48ftbptItxO+DAGi5mRICMGrs4oRxx4gkwwGFUl6iRDiMpkcxuVNJFdUzLlv37wP2ixVZfsZD05JE67FewmgMOACM5vgP02EH4uwczR2/DYc1/F6tIr9neVsUTLJ7NrDCcaDcKmJDdSEMx+M24OdR12VWqIVZNy4v7/VYzane5lWu2MIUtc7FDX4Wz972x0/C7s9bizpmuz84SXB+k6LlhRCWI8vDzSuRISpRfJiSvK8TThNAezXGE+voE+bWmvo2Cwtn4VrfqWHLef+g8/aowez9eP8geROxBl2KBYsW2UhevLUMlNUbxOyNXyF7wW7z1OqwoMI/WhX/mhJBZUgIX3BIv6qmBXWALe0pPuH5tXyf+dFvLH34L7P/a3SIYNDZxMC8F3TMnxMwJDDPK02m4Lk0wN79rmcFSsPHfXWePYYkxRQWnjME63TJbHcKGmww+I3bp7bbNv8dz83jJ4RpDQriSvzZEv+QxU105CMNvpoU62YOYuV0A6V0QhVxSIwQVniljz0++jTnIGG24NE2ytLmN7ZxXpwRA/+1M/6R0d6MgydUmVbpskiBARchl2bhiZxeduucliCQfWKckjs0aNOCTjN4/Ub/3iv08YQrCaIfhhu2GPYa8RAoUDZ5JvO55aodnroDZ5E557+CHUayvyUoOcR+FhJ0LtdudHEVMW0N8xcgFDMKk6955t4i15Eeo7FkEL57zvWLyAH9NZW0Q5bWMtu8a97XD2wqEZQZtj8Kny7EwFEqgcYdVWshTqn0V0NqHuw5C/njMiZrqQQy5rxREZr4ztscojGQgf315dRr2xjnwqg//4Yz/ila1dLSQXJgoNZJfFErW+K9FKLNp1EBs3pMyRNufnGZpsXj2/mgYGUh/8T9+nKk5WPoSBskm3zJDZM8szx1dzZAylYrhEqtLmxLV49itfRLOxpsExqWDCYzsyYL4g9wVRn5+ntgjnKHZbnoUEASOSOapWGUZb4kv23MEVLTpBBu4cx8/HwZH4Pr4K2Bgj/MeCh6NmKt18F4Ieso8Ou45/TuPwWD6XLig0Yx6/n5D4UGLnS5RLJEZah0JmyQrZNDZXCRevo5jJ4Sd++AcdLbPuipayNAdTIIwDMOGoKUHkfsS4mQptFlrMwBbWirtW5dxxsWUPnPX5tZ5qEP/dr3fyn4Hz2o3suNDpY/KGd+Lxzz+AixdeRNY9VO5wMk0M6SJD1CoUgjhnHja9cgM1DB40ocupoJBCZa42Q6qAT0cPOQb6K+4nNjDWqoPPFQscKjoctPHnDOctBM5UqAmVFbfbDhnVTHmZrqIRvx93eIoOWybHDJChXKRZFyc1hiafvdVGIZfG9toyavUNlHJ5/NSP/ahrNIIO1Epm7zkHyi94nbnh6bYfd5MlZsi4uagNhNx5HkB22pHMqC9P/ebPvz/hgKluwhGKna3p9fAodpOBdmzlZIxKJgJanT5Ofv2343P/9ABeefZRZNJUw6wVtvJdAhGhsg0T52TKuzDKMLsVhN11hEwqyEOvcDYi2c8HkkMXjXr4wKL5WLw5WgDPzH2tGh/f9eO7elfr2K6WgIAolJVARdGinM+BJzBYo6XSHysglLOWNgHJ5stC3bhjudDKQPXbqG2to1nbUi79R37g+1+jrYLepDVx51g5ctcsMUYrLdrtLxsmRqGqGEAUxF1QSprhN37ue9VAx+LBcFJMYsxT3m2foR3mHYXDzhK9ajVauO6d34Gnn3gWzz/xJXQ77NhgHuHkpBXDGxZuVRoR+1kmJ6V8dixQ5K3lhHmMKiKe57HNSfOiAW8UQGecjk/kt83W72a75FX/bwraQ+XLprmDE9/H5JFLxvdxh4emkJD3jDOnZxqShWPv0SKl89o8SOeQVTtN443xvflsVqyXTquOublZfO93faelI51PF4Idv4tx8e/jYwuTE8JhPpDVltNB5L2ClxDzl/qVD/w7lexavbEjVGNNVqN6kQ8RN+CFFhYWwBYQxWIeSSaHzuQJnLu8ise/8KAexpy6IeYXZ71wwOyWhVKmqqimVNM84lPvdn+IQgOOje0raYMCD4/sFheedj0ctkhphoqORY5F3Q0jvZPDGGWY4+JzRQgY6jBaXkdnhQA4ct5zRmgZm+8RIVSM7w1o046sSWPSnzVGSqrLxj/b4udff/11+OEf/EFfbGO2hJNq/lHAqJ5p9HZlaTmHDDONYxa1cdS6mltH56h9ogpUc/BLP/OdymczbolYkzsnVGXknMnbYq8RPvSo1ssTCCwZquX24NIO8MTnP4Mrly+OgILyBInwjEENFQpEzXZL3hrTpq2nWBD+xu1sOGJmUkIhW2Jf2ACT/DExY4iZdp+XvgYuEJM5vtPDHkc0EL5DaAIrKjRGy8jR89BHvVy8dZeySwlZKabOuU4K1cQxy6g0R/dXjqAuuPRd73o3/vk3vHdMjTMnb+2/FPJGaOpOqXnf5mkr7aww2Xh9Rllwe27fjHiC8WypX/zpf5swSJeKYTG351S5uATuc85bjpCF8bEe2u1jmlNNzzFVwvnuNB556LO48NWXkMomyInUDiwszo2AFAvx0t5vu6ydHdpDu9ix8NiNoY7DpBAXd1/JAIxUImGx1N5uY55Q5fE1JinEJa7Pn2PXCuN3vH40qeS5ec45FtxqoS29Glg2+WEquqcL7tGCqWAjTrCXaTTwEVU6ncKHPvQhlUiHmRPbhw7pWBp2V0CtBp73NQ3rFC0nMHCiJdzeL2a0+B45aSwf+In/OyFXiv27SbpXB6IRMS9tOLSyLN7wLpIQUYutBu9ZdIcJznXm8ORXHsa5l55Ft99GOrHWUlNTE1LZFDcurrzMPqE9a0jL3msGtJiHHwAHB8hdoqY3rE5UV0Dz3G3X7qpxg3stsRI7OhY6zAavN55wGXfUYnF31WhMqoFIRtm1/IBSvS41I+dJZLY0uh0nGoYdbvdUkkP1ru5L0XigVMQHP/hBoYCGVnr1ihMTuKjGOHGKkYeD+tmTM0ZiMAatSIteVGkIk7FUhcwpu5hC6o9/9/9J1HzVS2eEgdDekBJM58JPGMhmmOVJI3EUiQsshIv9vAg2II2vrnbxwvPP4qlHviSCvvBqVmeW2LzVPPKYVLOPhhoV8+wRYrxyld96OBOLEwLAWnH+jTtZsbtHBru7w9E9j+3Gw6zxRRy/7tdqgLh3CA0xcj4rd4xahgRI4YsgJ4222Om84deElookje1QFjQaF+/EyWvwH37sx91OBxXZulOpfwrDWmbt1FLL1HIIp1KqhRyGHWeiOOql4zjU9M+aBFohgiGRCls/9td/mBTLRWTUSwQCBZKEKTfr2zGi73oFQ3qw60QpNEmxwRtj3DSu1od48atn8ehDD2B1ZWmUiy6W8ihPGJPFvHEvuAtb64sbPkOYknEHSw/oD0xvM4SGYyTGzOvGZHxtDB3OllKKXgfN7yMBIgFyGz+uBew6VuhOSFRC5zy34I0x2aNIIW190MI+mgOaRTIIO2u5ezstIY1f//VfwczU9AhsspbfFs4JKQvbzHvGbg/AhbaakYznrpW/GrP1u2RM3ziujVMPff5+IX9q0KL2y757vGwm3H2Lei0nPY4hy6HxdFo/yeHxVy7jSw/8Iy6++qKpmEwa+VxWhQfRp4XccF5OdUjFDLpt6xca6pkTHs1aaU85iVTz47tw3KabJTPHJUKRWPiv1RKx2/lc4/cct7OKSZ0gEOxPYeXBb1NDH2eQuhYZjzLsnhmFWeY505QbCklG7Xd/93fjDW94nXPw9FcRMGge4h7RrYmXFzVpnA3rfPQe07DUKS64chIpcKo5G8rsGcnRk1kPP/JgQk/R0pykYxqYMALhnWLbb1uXWz6keeNx8k5KD8JS3VyuhOcuruIrX3wQLz39+AgUoNQyfjS8mXnznpAhkeDTAyR9CxnGqzPi4aJOy0AZE7RQw5EsYYO+r0XG4vOhHcIPCDX7tSp+3L6H4IzfS8wVz+Pzmv2ehakhMCEs0cFR3HkdTZHHgYMH8KZ77sGdd95h+RWRRUwTRe6BZkkOn0cQ0UslFt9Ewtil9PLDWbOMJVG0XWbqeMtt81E8qfT5z9+fsBMv7aHVPRmfigNSAl0XIqmcRXQseLOeXqxgZH5a2DbhTZ2pUcCVtW18+nOfw/NPPKLUpXUpsm75LMfhBLJVRKdjvcJZE8XidoUT8jDNQYtJCE95F3TZ7T8mQqEcOscH8plRV4TAv3fBEXOc+IpESahsmYgxtC3MQGiPuHcsfpiC2P1a9HYfe/fuxfu///2iHhsM5Pdy+rAEMG3PZxTh3TGxr7uIEuwU6Y3reV+WRRlgYk2AeS91qnAiYtC2rJWJbRoCQcIlIivorcVSD372kwmzVjqRJ2vdh1l7FQDEoGt4axSuST2pgsT7blLd+SEtjDFT6QKefOUM7v/E36Fe2xoxIwnAWO/SrOq2u11SZ62WizaXLzEyHXCJiYoJjh0+PtFy1EZJGh65YDZzHIXiIkZIFRBo7HK+N8xULGjYXA1ojIgYAjCeJ45dd8cdd+DffNu3e67AKjZpQ6PG21SpF+2JXGmYugmZVW8QhwgnkjtcvD0nDHLhtHO9k4L5GAyTdxeVi22JKzp0Rhahn0EBoGoX+vfpf/ibJM3QqdPWLstn85icncYLzz6FYcIwjJBnFXv37ZHtaNU3MUgySGVYrZlHZgDkK2wIYwxPqphXlrfw9x/9G6wuLwlDZ5E4ww+q6Xqt7g3r2BfNeoMOKInOlFEI70kRIy8ECXG3VktxtZzH6LliNnZ0ksAYOTGw5JjIWAC+N6jIdoSUYf29riF8/G9CbdpGCQ5f/NAEHCfr2n7mJ39KY2ZhgHqjD/qqTbfEhqVbWYynpvYD48rzFa1GuLBEIlUbzoZ9Y3kBnVDk7SrDbBCNMzqxaYg0mUHhs+ikBeMPcvz0j4zFk0Lqr/78D5Lq9Ax63bYkgdX611x7Eg/d/wkcP3EKi/sO4+WXX0Q+m8aBw0fx8tOP4/ipm3DxygomJyZw6dXnkJ+YQc/JJCwiT+XzuLzVwSMPfUYdE4kzVCtV84QdoCB0yvBASJDiCqtdGn+Zat/9XahNBXoKKSJDZHlmkiNjUUMtj9vmXe+eMazVnekeHpoY08N7sPjC8prjsWqo0sgw/b8/87OYqU6pw7HUvldi8Hk4FoavfFajEVGT2PtCg9gzMS9hVCRRmdzzj0NtKDChUaTxmPpVBMDuzz2rvuUpB+xVquY6lofv+r34GYFVH/nw/0hm5mbVe2t6egoXzp3DnXe/Dl/8p0+qo++RU7dgmcXvVy/h+tN34IXnnsDJ625Coz3EwsIcHn3gozhx+s0oqEVFHfv278fTX7of5cM34S8+/GEsXVpCPp9RO6geC/ac6cLJ4aFkQnpiQcc93rGFJl4VvTsNVCHQE0wWS4wYkGKCQVNjDppXcnqXYOamJQyBKbN6xc/90G7lzus6Bz1Sq9EiOrEMHR1F64OSYHJqGj/3sz+npEh446ERgnI1KgOWX8IerB3tYIJNpkms0Q0PYlPNupMuIoyjsLIxACneuXzBKkM8VCQMbfQuo25Rm/R40kGpKN+l06xbXThbpdCGs/PC3MI8dra3MT+/gLOvfhU3n74Vzz/5KNqNbVx7+xsx7PZx5sUnceTkDUpyFEtVzC4eQnlyAk9+7mOYmN2L/Ueu02IfO3YUjz7wcUzuO4LOsICP/t1HUaMq8dZV9DKFJMkeGUU2asis04QdTmbVIl5HNebIjHunEarJ3ku1pcSQMTVoFY2aPDXX3c1ta4d7VYWS+4RMM1YjxYlnSMjvdz16i5F5P3rXFk7mVaX5rne+Gwf37hsldsLBJFeNY1LbixZPTjCba9i4naQQfk803+NX7sDwJaiGubhsTBC+C7/yOjqZIA1t0si9B6N0e3vHyCNk/uq4Spbx9pD664/8fjIzO6u2FWxNwSTG8ZPX4crFC1i7/CoOXH8bFucW8NzjX0B5eg6TlUnUG01cc/I00rkMnvvypzTA46ffpAXau/8AXnziATRrNRw59UbMLsxic2MLTz76EL789BksXb6sXWGevrMynMkSB4lG191oWZl4q0h+jhQqPgiPfeAujxYUVu/sPcZGoIsd8Cq1SJUfdc1OiJQqde+fAIXh60Md+CoMWiR9o/bypTiYcbP4vEAubQ1riO2Hz3H06FHccMONygqye1TUG/EZFNuzOW+vp13ISwVMSgRRi+LnpfCrteMsqgcMhZj1d1w0CZu34OTOpkIzSDnB7MysasXYnSoO4su62Uj99V/+j4TF6LWdOqqTVaxeXcbhoyewvbmGK2efw+yBa3H0+LV48ckvoj8E9u87iq3aNvYdOI7iRBlfffJzaOxs4/ANd6HEHT87iwuvPouNy69i7vAp7D98rR7wxScfwKByAB/72Mdw+fKyqb2BdTgO+0Xpj7CEoQapwnzIyLZx8Ny1Ukm0/Q5YyJN2gbFsmLXVjOI4LZYxHV6T16ZajyTQbjLFD5rLG7NVbBSP7y0c9DCR2kQcNW8G7zn3cNCII3CcLHZg/7SJsp1lwrCM5nHYbSmKoa9jdKs0+sMu7Y4EgYe55Qs2N9T/1g/V6r7Y+ULOGokjjZqKKNVpiTVfbPbXrKPJDlM6Xbfgba0HSP35n/5uwqpEa59cBM+Xmp1flId86ZXnUJpawPEbbsH5l55Rw/mFPYfEpZqc2YuFxUWce/ExbK1cxsTiMezZd1iLvXzxPNYvP4t0YQLX3vI2dSB89bkvoNnq4vMvLeP5xx8fqR9BmNHPVOwV271c5JKfFMDfaZFzu0kaIWV+Qq86D3i2R4APTxQKh8lLYwngMOHCtKrRjiyhEWaBqcoAddQtSr3COXF2hgfbVZl9NB+DZT8sMOQiqZuTzibxhgEOdFBQeF/ZVPfCC/kSDh44iONH9mNl+SoOHTupnnArK1dRmShhdfmiHK3DR67BytUVnXaYKxZVhdlt1sVJLzAbmStg2GubZnNIt1CqamytTgvVShkNP6lPWolz9Vd/9jtJvkxyoDVutzjVmrGtXDwnZujJG2/F8tIFbK0sY2ZxrwSjOr2gU/GuXjqLnaUzQLGKhYPXYnZ2Adubq1h69REMBykcOf1mdUQ899LjaO9sYjs7j4985K9Q11FN5pUyZOFXWtp9+/Yr3hYzxI8nZlTGn6lo1ZMz2l97VaaFFlSnFk7xWlJvcaY2QaOx46oihqeaFN3XF5+2UPdxhzHUvFKq7jCypo0aYZzUEeDLOFizGzNb7xQV5jmGoNjeyZgEnt56772YmpyS8DY2LmNicg7XnLwJly+fxc76KvYcPIyt1VVkEx4ydxUz+49jbn4R68vn0ajtoFouQIfjFLhBymh3Gug0a+i1TdAIdnE+Un/xJ/8lId+Z+LUC+X5f9pDhQH19BcNUGvsOn1B/tPUrl5EpltUMNpUpYe/ePdhYX8ba2efFtZo7eB0W9hzAsN/Buee/qCMo9p28HYcOn8CVSy9j+/IZJOVF/PnH78eFM+fQ7Rnezfvu3bcfh09ci/m5eeRy1sEvuv30O9bnrMQDYZx2LBXrP3Px5HQZqXrk8Qu8oPCy+I5xrjea5zPy89FFOECX8URKNKoNgYmkCSnBStHGkY9RPDiWw+Z4IlY3xGs3JByhdrLhPF/T4F8ybCmQxw7OYX7vIdz9unuwvrKEKxfPYe+hw6htbKDb3NKc7T16E0rVKVw5/zLQazGzquKLfGUGM/OL2NlclZlg10rejzSpEos1//T3fzkR31nF3XYqnzrRF/LoNJuC6fbsPyJbsaZMFoeWRbZYxsL8HkFzK+eeV0gxufcYFvcfE3l96dXHsbO5ganFAzh6/BbU6ptYeuUZtb185lIT93/606jvbKDR6eOHfuKnUW8P0B9aX/B+t62meYwfCXiwebwWiIiR0CnGqhazdhjX09apM7E1j+VxVRFeqcpFaUMrciAwRE1g6VaDaMPTDR5XcMnioNnIkAmNU7WqMWIDsKHNpcPJ8NLOFfXTdrx8KFp18/ddnnnqfcfl7XtmXGeSqZdMTxSmQwcP4Z7X3Yna5oaAm15vRwvOse+95laZ3NrmEmqbV9H1as7yzF6kszwQponWzgpSgz62eYpvZRKTc3uQ+uPf+/kknS2gQM/RWQ18eC5Kp832WAkmpxcUpNNpo//KTZUrTmDf3gMCA66cfQHDfhPpyjwOHL4OxXwJaxdfwtrVcyhOT+PaU2/ULl8+/6zUYbtyBL/727+NlbU1fNcP/LjKaLa260ilzYwQwKF3WSa/LUlEqqCw8RpimGZJY2L/MaYQ+xh2efRCH722N9cbU8uWGrXr2kIbYNwmsqdG+EaJChiWX62Az1pYRIYvgI02QxgnSQaiJWqSw7KMcdXbTYV90aXJEiZ23rbF/vZ9HMhqHRSkPVRTwTH1UC0V8N6vvw95HajXQnNnW4zUvcdulTlbXzmP+tZVdFtNadvS9B6Z1+3NDaBXw9ryZWvik6RQnV1E6g9/62cSNpnLuo1MeUaF8KBaMOoQlylkeUh3r42GmCZZtdCYmJyRyqfdbuysI5cvYe/hU4JXV69exOblV8XeYAjGU9uvnHse9Z1VzB64Dn/2N5/EiVM3Y3pxn45n1IEvLEFVKGPg/wghEzrURSGbt3M1szxkhXGmgShpgjE89LxnXYLZs7TXZN6YkGRXNdGKad37p9dPDRKN9tSvLE+wYjCCcFlxysW26CCl7gahBfg7zoslM6xsmDvbnD5r6MfFEA7gvcKjC4Oa0PF0AF7DY2p+r2ILfc5r5HrWFLA6kcc3vOPt6LcaGPa7SJcncOyaWzBIp7B+5Ry2rlxgcY5M4fzB61EqTmCYdFDbWMba1SWFqRSwyvQCUn/wwf+YkKhAiaItYvsIhhNsXqf2Dil6x1UZeXYopoqU9BdLKFen5KVurS+hV6/JBMzuP475hUX1DVu/8JIWYM+J27G4cABXzjyPVnML5YlpPLvcRXlmDp2etd8S89QXkhk224l+aqA7TMzMyXazl6p77oasWSUoEyqceDaHS3kbCi4YPVnZzYT/DeumqdFB65HedWKAWlzJy/YjLbwgYChTMlCOOrSAOYK77BtpAbD7RFvevPkJ1pGY17TkhrUXCdqQBMd9iPBfDDJmVScPaAW+5Rvfi/SgZ+ZtagYHDl6PHoZYv3IejbUr6LGWPJNBdeGYmgT3ei1sXL2IAR01xuoTFZSn5pD6g1/70YROGNtIkFrERVZK06sp1JvDKx0M+7W0W5LKYnJ6CplcEd1WDTsbqzqFoDp/AAcOHlEP1NXzz7PfFqb2X4vZvfuxvXYVm8vn1PZyYt9NuLTdwOb6ttAuJUl27LhFmgp77Ta5s7DL6sO5s4lghSMU5bWMyyWILhQcL71QCpESFd6ey0piTCtQGFhTpSMn/WgK4eXMoHmKUhAoETcJgZU80RsPx5Dawzh1LHw0UkR49LxnOHcBgYawBFrGnyk00gxjPVzlHWWzeM+9b0C1lLPqmvwk9h44KlOyevkVNLau2rNkM6jOHQZDO4ZrO5uX0anXrCd8Lo+JyWmk/tsvfH/CKgZCRTlWIFKUrNLLzqygM5GyKkURERkzisGWQ5GdFgoTGPSaaNW20Go0QCeBi02MdvX8CwoBJhaO4NCx42g2a1i9+AobV6By4HpcqvWwvr5lZaaqELWJ4iIrJednafG+ERLxIQmSiEbknCum9Pi5qNfm7jOWqhMTiaDpyGg7tkH88yGUk9fnlIywMLA7sG4S2ZQVshMjUNJDXYzICvW0qHvhhoFbXpq7qOskD2kYp2AFeV+dFb6mTCcSKiGMwaAJX4Ff3/2W12P/4qzWZXrxKKbmFiVcq5dfRae2au23CnlMzh9BuWTtvzdWz4JUETmZ6Swq0zNIfeg/fXcigqHjyAmbzbK7AltLyzYzCc4qA3c2VFCQIJPn+ZhF2XpOXmN7045xqlaxsO+ornHlwsvoNtaQKc7iwPEbJCjrV86i3+mjtHgMm/2iuFRXr1wxRMhPD7BeXl0hZOEpR1ZMRx555YUQLSpELz5Uk9eoBGU9eJ4q11RmxOKWnuTCkCnCyfDzNpyDprM0WJbkvdA73ThegpSfFnLUbqQww05D4PUUQXS6fta3lSSHLQ8nLnZ34O2RJo0jKFyVuYDasVFxxOV77nsD9sxO6muDMwAAIABJREFUSkUX5w5g3+IBLeLm1bOobSxZGXRviPk9R1GZmsH21ibQ21I0pANwGx39PvVbP/sd1AFyoDgwNokXu8MdDJaeplM5JDnLVVN9m9NCmnAJ7A+mZCNVx9YWUrk8Fg8eEzy4fPEVNLeuIElP4NgN7kEunUW31UV25iBa2WnVSa0sL2uRGA9zt6lGKTPEsD806JBN5ssT4IlEskHecC8otOwWQc+a0Kd2ijxj8uDN+7bOidYWK5L+dK7YYpMTpaSHs2aiSWyUNxGv5vENwx6dKPY86arUNpoXtPtdMw/eKIj4dajigIEjPx8xdhAX6DyFoxhCbQ1sR2WaEuy3vek2LXapNIGpfddgbnpBuYzNlbMYtLcUmRQmJjE1sx/FiSo67SZWll5B3rVVNlfEgIWHH/rAdyZiOaQtO5RmGwmiUZ6xIQKsGmVWJqZTVmzOXaiOPEWUJspuuwaob22LZTo9u4Dq3CK21y6jvrksFHnx0CmUKhWsXTmPZn0HufIc2qX9SkRs7WwpyU71yyOQAokKtRyn+ubyhosTdaKNJVOTqUL5QGOlM2Ez6UOojIZwqx+uqkn1BjTMGFEzWJ8XClZeuLLial88xqqETOkEqTmfU5iUVnXnyrxpO4SdziCzXJEAEVbujFad3R1HZYjM4Od8e8M6TmQc16gx+CE0//xdb0KF53snKew7dBIL83sl1Mvnn0ONNps59HQWE7P7VRde21lDNunIBxLUW5kStzD1X372OxOzOVb0zZBLaFTBHDX2CleaMLFQQkcTqNk5Y/Gy7IF1sx+q9zYHWChXMLfvIHrNbaxcflU2ZfHIDZiZWcT2+pL6irAJfXfqGvkKXGweDcFqTsbtUaHoLbSlVjmZhFE5JmLcUc9katGQNf7nwgX9iMQJ29nBJPXKEYV5u6fvMU896HfkeCrP7nGwbDeb1PJ0wFJeKBfrzsLDVt83liA7kKJkhjtYTGTQOYquhMYPYzLeqFfRwcJy7pGPtwaC8iGcEcr+qd/yjW9DliatWMb8PvO4eZrP1sqrqG+tWPuNdA5z+46qgrTZ2EK7tqbjP3QC4YB14hWkfutnvt11hpXQBhtEh6MzvFExALnZWaTzVn8sJiSTD7Tn5K3xZKC8nYqrcy1KE5if36sdtXb5FbFVJvccxszcgjr4s3mMSIvlEwpVOmxDUa/LuYlcbuDVlvWx8ETd/dkf1Q84CcZKwkXgJDsi1uq27TQgr57kLlVhuoTaGTHe2sPOv+buMz67cs6eCrW4Oiv8nCRJOX19rzrReR5RgUJBs8pSMkeiEQl3KtOl7CYch89F01i69jI3znc3X4MttqzDAgWHWmeyMoH3vO1OTFan0RoMcejoKVQmJrFT28L60lfR7zYFnKTSZWlT9UEb9pB0G1hauiRNUixPYDhII/WbP/2vTY37ohqldRdW1NmWKo/M0OCpFFUYsnho1geMks42URaCMITIozI5h8rkJJbOP492s4nKwkHMzC5qR+6sLVviYvpa9NgxMWV8rJ4X64fHysmXSiY1iBAn04I6e9MSGNwd3Fl0jnhdlsFGaSwFNc77oAqLuF2qUud/GeOFcTX/RuFmbRuJAqq58lBqBIl6fM2TiMPmmrnY7aYcp/Ba41w3LXQO++yVZJTrqLSMggdreGMLLSrx6IjqtDTD1FQV/8c736S5nZxbxNTsfoVXPDu7sXEJnXZNglyd2oPK7KLYNIxqCKrwpGSmr3fqdZRLk9zZ36Fi/MjcREDPiVD44+CCtX5iC1s/c1pnhDA+ZjuJtJrCMUHP9BxDNoIwk/ML2GKXgc01ZAtF7D10UiqPP7MNZmX/ddjqG57MhHuj6Uc9DW0RR6GKdiorTzpIuEu7hpUTEVP7KLbS9J7oXLxI6PBZomCdpkjtuHg3jdvqrWk+goIbTQLkoHq7jvGwyey9dX7UGVrcJN4dOUgQ/MoIYLz/anjaUZAoCpXrU+5sgwGN2B9IG1uAc17vufs0juxbtM2RLePwsetFaNje2cTm1XPotWqoN9uYXdiPdHZCm6DXb2NjdUmhqDUw4Jrlkfq1n/y/VJ8ttTFWlmq4MGucrMsfU53y1kX5zWHo3QJ1oEqprF1ON39re0tYNosGipOzysisLZ1DtlDC/P6junnS62Fnex2Ti4exmSygM+Ahbzy1hhMPdFpNLabSrCsrQsbUUbHfwvbahtSikKiehU089ti47XZS4Hi1pdGS/MSByIJleaotbbkVHhi4stulwPhscYCLV0+6lpFH7WQ/2d047H3sFEE7etF4YSE0VmCw26dVrFvaZTpq6pC4W8BHLcCzWk7fcho3nziMTqsmBK5QncUij+FImGhpY3PlPHrNGjvJoDqziInKnO7RaO6g19rRQQHUVKRIsX9b6hd+9F8RNbbzPoTC++GnnguWeo/KSTVbpUfMHizehsIPbGOF8GR1Uk1pq1PTlldOpTAzN4+rF8+jN+xg76HrpHImiadfWcLk7CLWM3tF9WFMScePue0aKTU6M2tTCRFmgsjk5RENje0dqXvBlElw2g1vHq9uDApSLLx2ZZza5+UycVipOh6JyMIODFGf6ScI+yLuxskegqrbgrFbuctD3ZN9kuJCC//uW6/vsb7qTGqIaDFioBikGqzVfDaDt977Nhw5ehS5BNjavKjsI9X9/IETmJyeQ2o4lBrfuHpOY6YWzZd4tGNFgkuKdrOxiWG3Y4fJcjMih9Sbbj2U3H76JuxZnEW5wGMgbGcYsmTHOUnL+JlVVNuSfB4xIftt8CV42MpE2equqxXtNDam3X/oEFaXltDpt7D/AFG0JiqTU9hcX0OhmMdw6jp0kBOjIzhZdNSIVtG2Moxpt5totWroNNtqkcm/G1drt8JDp+xSCBMoHAv4MXaptFLWIFYdqRB9x7UQdppwf2AkiqhBD7ttTiNtOyfDW2RFoTyv56Wz0jKEPcWMTsk5ox7ghomW21UeLyV2ib2OHz2Kd73rnTrakX7H8089La0wOTcrz7+2eRk7W5tqaLD/6CkU6FUnJG3WsL58Fjwsjru2VJkBUkZy5GIPBy0Mve1GVwfDVZC65YYDyc52DZ1uH3vnp7BvYdKci2Qg7teeuTmxKKpVghpMORpRwFgtwqasFbPjuJwoeucKHZIheEYlJW91dQULe/ag3e6iPDktQiL9vurCYaxiHgl3sLJUHaUtZZO7jFlbaDUbqO1s6G+M5UmOCOyZE0Shi1NpFaOn2bynjEabJTNZxc/WoZ+JClOlPG6AgsoiCNavjRIgsJpoU+27rUWCjCDVOxiiFGd48z00H96TLCNUz2JrhWR+AnAqm0elmMVEtYiDC3tx/fU36Pip8ClUxpMCnnj0EQlloVpFv9XC1tplgGeDF4ooLxwWKbRR20aztYN2bUtzRH8qW6yiVK7aCcHtJrrtJhKCQATApE2ySH3vv7o3YTqvR8eDXYa9+ZyqCr0/mb7qRAErLdGBLf2hFnl6ahJ79u7RQSqGaLGSgtUQrGe2Qv04TqJa5Yl5fRQqVSFOxL6LE5PoVo+h1UuBNWeKibsdLQ4dL8boGxtrGrg87xbP/zLcOcJEqWOPkYm4EeUSEZD1awXrrM+QjQfAqgyHKFjBCIUsT2ZhgEgDNGEeOAU3OxbZ4E1r0MvPTfL0PyJnLhhWnsPr28HqFMZKtYo98wuyvRN54hCb6LR64gIUJmZxww03jLo+EKmjKfvyF76AieokSpOTWuy15fNqbstoZ/bQtfrabtaxvrGiEJbRMdkz1akF7XpD69qq8GFYxnFIjdP3+vkf+iZtEjZmV6rNCXW0wZwk4b7qprRbtald5z1MlaPyqg4V+fnpPTOzM7j2uuvEqCAIYIOwDj4E7SNVqQashTkkU0f1WcbqFBR+JQOD8XOzuY1+u6OfyaYUB9pP9RXgIgDD2leJBOAn7vCe6YxVTPa7BF94CkBJlaOBgKnvJ59HqVbadfNfmC3Ty7NbnFUlJzy2Vh8G92tYp8Wdye4Kx48dU/NZ1p2RYXLoyDVoNxs498LjSPptEGsvTC6iNDGtkwXjUHoWPfL5udiV6pTCrPWVZdRWz9uclWew9+Bx45HvbIrlQ4iaY2r3eiiXp1Am7yCblT3vd5mOrqtdds6Zralf+YlvVehFhUz4Ubli5oVVAdGjhTJnw20UmV4CKFxN8fd2Gp1liSIG5c6k/TLbbwT9bsfO/5pfXJQ22L9/vzx3kh6Ge06LVkumZiQSqKLIrWq0ttDheZs847vZsF2tQ8GNzMAXcXsKJl+BSRND77Pdh0jypFsVBcwwNOFY5ZiNjk00Z288V82Ja+zU7JgI1rn5ATlk41II+PXUtdfhmmuuwebWGmZn5zAxUcX66jIaNfLF+rjx1rtECrx85ln0W3XNyfz+48gVyzh06JA0DL3xKGp89OGH1fF4Ye9BXL54Dq3NS1aDXZzGgaMnNY9rq8syZdnUAM1GU2dwZrLkBvoZpMOekk6N+rZiciat5KP815//ziSqIuwQUivoppo2NTeCeXczSqPOu+pY7b834ELagQkJP/vLSkkNmaOU8e+0pXSoKCjqMcJMenU/7nnft6Pf2UGjZWgWsd3hsCe8emdjw8kTLQmWtWvmrjWP02yxOZb8T4I+zzmhGTFP2QiJKrLzDglBPxpRguh3iOPmJ+QxqZKy9GppghqqjLfde69ds83zQbMoVytaTFasVqozow5Q3HV0Lq+/5Q70Wh1x6evbV6U5D5+4VZNPPjmdVDsdyMptv/DQQ5jU4Xd7sbWxgtrVc6i1apicP6bUMcda49mpTXaeaongQLw+V54VtVspzWSI7Y2r5tekmYqeMELGf/9F9kET3OMkPe/d4VxsoWVaLMNwhdCovYNpOU2hkhCEuaPO2tpRmJPDybfLqwGxeox6aa4awQzVpyWXTuPU130LtjpsoleX3SNEyd5xW5tb2FhdQTLoOH5uxEIuaqdDLNwiAnnebPQeDVr7xLG9/4rCoYHIlJEGDWhW2pr0q4nyqE6d5ufmm2/GwX3k0PdF0ZXjxRMH+fBeU85Qi1jC6soVHSBPUn5UuzS3N3HkhtO4dPY8Bt06NtcuCTy68dZ7sF3bxpEjR3RSImFTWhCO60uf/zymZuYwNbuIrY1VbC29it6wh5m9J7Bn7wHVfK1dPS+NOzs3g1aTMHMH+cqsauTps2ysr6K5sy56mBrv8Yhp+kh/8ts/4H3QbCFUye8Hh9mC+lGAYyfDKhRLeeMcnbgzVP438F1CjwJivGVlnE1l8pSo97ZMgxPuGPqo9CYzgeqJN2qhGVq0CBgM+qpDI6mOtCjmzDfW1zA7M6NDaKKihF2XVP/k7TEMJCGyV1S8ywklXYgPTRvLF0/lLZQKKGSyuPGGG/Du9/4LhXWdTl0EfkPlGBV0lQ3kiwwcqnU+Kz1fmbp0GitLlzC7Z49OGZC6L2Rx9cJFXHPtdVheXkKqR422g6Tfwb6jp2RCWFBRLtuYTY0n+MKDn8P0zCIq07No19ewdO6ryoQdPH6bPPJOc0sHwHaHwPTstNLK/V4TufIMZmfmNa619avi3ak8macPq8Chi9SHf+dHRottIZf3J1HHwziT2k5mGLEhBe0ZnCreGp0kPyhUjEo/RMXAA5oDU+8Ww6Z1noaYrN7OcgSqDFNo5efQyS+g2W6g120pxqYd7zQaaDV3pKZ6ZL2y1kq4vbVfZm7aTtyzXR4ghQANP6ScEOTMzDTWV1clnG99y73Yu3efaYheG7fd9WbVk3OxL1+8LEHrdpog/6xcrSppEW1G5Cc455sTWd/awMziohaRqrY6VcXls2ex//BhrKxela/BoorlC6+iunAIczPzYHRSqfD4KFPj1C5c7AOHjomHT01QX19Gq0Ou+M2YmZ7FkjgCqyhVyRGfx/bGhnh9E9N7MDU5q8UmgsYTkzkHC3v3iU7FRj+pD3/oRxPtwniZiR21QTYQwc/zEp4ah5fa7uBLB6V6laPgVe+sFDndKGS3YwYtAxSokmBFaQ1ChoYuDZmTTU1iY7OJrfqmKE47m+tsrYB2py6An+8jt9zgyzTyaibIrhAFUW/Z8oKeN5242s46zp05o5OD5YB5XzPrMgS0egNcunwF/+67vwf33PMmdfl/5pmnMTc9qaggSn051kbdNAjPqpYvkIJUJ/GAyWpVOALHUSpTnW5gbnYaV5eXsdNo4Prrr7fvazu4/ba7jSY9wR7ljAKsCPHBBx/EqVM3YG1tXdy+2uaqophD192qg1fPnXkG2QSY2seESB61zW3UN1cxtecgZqbnVQ1y9fIl60RZLBnbKE50+JPf/qEkCgREY/VWjdEPk7syXsJ5/Sxt6/tlQqKe2+y0pNaNFAw/US96aXpvci66drtfUI4Z0SQ/F5rHJUl4vM3ygWtuxeKho3j2madw4eISVq5exZXlS3Lc1Bd1dhYnr70OxWwa1UpJMXJc3zh4ea8qoZcgN13OA3ciNYQa1w/TaPUH+PgnPoFbbrkD//7934/6zjr+/u8/gce+8iVzbPw4BjmTxKjzBfHv6E2fOHlCLBoVEKiYzzooMKTiTQnt8kU0jZWdWyR4qClRWTa7Up2wolB30D73uc/h5MnrsHR5SVU4w14T/e4A+07cjG69jo218/IbZvYfFBeP8DFbWk/M7cXePQews7OB2tam5fRlwzkHnpn72z/8aanxAOwjTKKaVk9MERVYrWidjvRSQsEWNGykcrFjjdnMsTPnbVxpWBtn7zzgxxf1ujxxqCTkSCfg+HX3n7wVB/YfRKu2jVy5irnFPejq8BlDuRhFMDR76cmnlOyQifAyXFtb4/AG6udDdxKenxDkDNLBMAfCive9412oba7ghWeexSuvvjRKDgk1pBZKLEMXzeLJsKEfEXRg3mNyakr2mKElNYyYs/W6wkzGv9RGrVYPr3vDG9SEiLmJhKnWYYJHHn3UBHYwRLtZUyODZquDI8euxfLlC+g2a3JoF/fvw8b6ppVZnz+Lyfm9mJmdx9raFW2GcnXaDnuX752oKDD18T/9Oc96xaLEQRu2IHTVY+G4+GKMyMZ46exoMQ0UiMW1isZd+dC1YrZdnYcNZ77ZeG86ZXOUATp43e2YmZlDu76NVg+45uRJk3T2YvF66VaziacfeUSTZbVc5L7HgY8mbAGt8jMqDBiZJdvsSln2SKIs4u4336MzPK5cvIiVlSVD8lhPXSAtyzo5jkwQixG8S6OlVXkd4tI0N9ZhgYJAweDPtPkkVcq5K07ge97/flxz5JhCKAI/HOcjX3kEO7UaSjyLs93E1GRF9fB0tLrNBiaKOVXDTs/PY3V1HYcPH8aV82dQnl4Qf2Dl6iWU8gVx0phfiDPAei0u9of/s+9sSyJwN5jjZd0LvARaDlks+rhaJy4rmk5sei/U293NVNbet2t0wIqfejvWEE622lmgUTZz9NQd4kqz9HRzcxu33nan6EN9LwgkiEsy4PNPPAHjjscZnS6oLm3xe9M+u2duywt2fjzbhPLnm+5+HTavXMH66gq2ttcFCAlhcx5ZtJuyyfImc+54RuPa2OWMAthjbhxyVeTC1hq9Pk6dvg33ft3XabcGBflXf/VXsb25hTvvuh0zs9PSIoRl2W2KHZwD++dYGT9rnaghU8DUzDQ2NjbF0WPju+iwVC6woH8LqU/+5S9rZ4fKDRUbReheyTc6fZ04ehh9U6XehMa98dHnojmNfm9N9ETrkZ0mxkwN63XVbvt1cLiK3kzLnLjpbhRLRXD38nD1O+96I5JhV8QH+ges/OA1n+VikxDo6dlx8zFuRsxRsVMLOOlW62VsWXK3KLQ33nU31i9dxubGGhrNbSUQQiEpDeu9xSJEDWaqJYeM/x5HJGqR3dkN4CoqRukLTc0v4r63fb2gz26jJkH8h099SpwAopTtVlPPvr29uUtXJmihA+ZSgqzvu+8+1Ld3UCiXlG2k+aht76hogI6q2Dre/Sn16b/6oGlXV8dsnRFVhoq7YWCFuFGOhu2abtsZHCQJDeEcGcgSoIqlEE2VxiEzpt9JXrTT4Omhs5uQdxvy9OO1N98tpIxNbzc2d3DrbXcDSR+dtpEWCMgQwHjpxedEpzWYNHaupSo5vjixwMa/Cxrp++iE3DcTdPr1r8fy+fOqH6cTx6DTHDM7mUDM20gWceGdzCAz5R0gomOSiIuuScRC8ffaGEijmcBb3v4eVXU0t9Z03ccefxy1Rt2Yq85eVX23OkuRjGnnoZHvTu4AfQGdlUrT0TUYuNu2UwtOnDgpp3Bxcd5qyD71l7+h0Mt2HA8xsSZpRKFMPXtxwKhPib1P6tDroQlUkJkSXXCDdWEPz2YzfmqdN3qLUMwOHkvbGWx8qQGvgTH8/ckb7/TzNbjYNdxy613I8HRf2h9fbGLNr778guwcXxEh0GdQBYvzxU2VjqnwMSxAdeCevrrlDW/A0pkzKmC0fqm77bkoKrTB6tbsr3EUTjZ9LFctyFjQoh3hZEJj41AkkCvjbe94L7r1DWytXpEwPPfC83aWp1pVG8AVTXEZbYRGMg1h1SnBqOUCc/HJ3AmyhX5uNc0p/cSf/1qiRQ1P2rsKEQZUJkdlMFbgZ573bvM3O/PKbqgDUehgSQ17LjgcNnfOwlFidkgagR2FoxhdYZA5TKQv8+up03eKSUpEbWNzE7fe8Tqp0XZzZ+R4MYw69+orst100kYayk/dNQKGTdiIheI2llpD75fmsTHfcMeduHzuDJo7NU0QkS2xXvzc6+C0x7OEBov7aq60820xdGBtHGrLa7Cu24PP3jCNe97xbgyaTWxcPa/fsuecAVCR0DGuqti23lvNSpssK2lA0mudYwaaIm26r0HsXJnLB//+vxso6lAmOwT7Jhsttv4uAiJ3+lj7Z1eJRtAzMMVjldFiCK/2npzhrTOjxsEqc+axLwWHfULMKzfu+nU33+HYb1uY8Onb7lSIxpZdro+lwi6cPydIlU6aqVNbHMX10VB+jEQYioQecoSOAfjceNedWDpzFvWdHfMxvADBivt3SUu249wshB13tW6pYkvnkshh2IVrQ/YRVTjIurIEb/7692ix15bPSdjOnLHjLWNnhjDp7G3vrhRahfehWuecGF/d2EVc7DA7ETnIdHzm47+XMDgfSv34PyfmaZF0UhzPf/RmMxa4CfHSronuAj6ZvImdOGelqqPJVAdfO+A1doEWX9CrxMkaqovsZ6f63va6N2Nnh2yMLlbX1rD/4GEcPHgE7caO4mpRfns9XL50CVubm+Kgx3LwOgQ4RlI/5liJTOiHoclPdDVObXP9LTdj+dJlMWnIXo0+M+HHBIEhTvIbuWxxGq6r6NGCeZM+Cz0t2WSwM88USeMt73gPeu021pfOCjc4f+6MLbZ7/+FjKKtHAfFW3LbBDGJVqYo2kB9O5+FmNCaK45hTn/rb31EMUSyzH7j5nYb5+jmY0TpSYZLtCd5InQ7Ey7JSHCMKGL2YixkQbOw07QS/VrAzQ3p1Yg6rJxw2NcnN4vSdr8fm5roQI+5sxuF33/1GtOm5wjQQr7G8dEU7W2fZOu891DMfSrsjcHkXKIVSLqD8W4BJR05cg621DaytXFFPEiFRHFsY9TFnVnVZrloDHYxdZ6cGBbRsjeN3Y347S6SHDO5953vEe1+7fEaLfe7Mq4rVJf5+T/lI1ppAOL11d6TZMc0YZA3RrLxvfKzVa6KRz/7D7wsuDXqNUYqNVmyOWCBj9tCjzkTqG8qdGylOs7k6scZzmrb7DR5VViv8Al8AMUIlheYV6+jBqCbVzn4TVtdW1FNlbXUV3d4Q97zlbei22KbROvJz0VZXVnHl8mVRbCOc0iLpQBpXoe4oUXeF+jaBsNEJ8k2l0Wy38cd/9Ee4++7bsY+JDR8bif969miU4/6KnWoQjFwzcdG3xZJAMbN+JFMQHYnLI4Ove8f7MOh2sXLpqxLKC+fOGiHSVf04UBU5i5G/4AUOfA+F3tg2u5z34BGYtkwj9bl//OPXhF6jvp8uwRZnGjFg1NGXUpqN8yzNSVMxgSNmYZ/ouQZyZuc8ewStE+fNhpla2z1wLVpPJEkGt73uDeKNE3VaW1tDu9XHvfe9HT0S6nqsDrHFXt/YwJWLl1R/TafFMl9GJjTeuFdwqurFgJAwLyNAiAxTb8BnThaBlK44dYahu332tG8cZ2k70M/T8uOVAjnUCX0yJxae2nvjUBrqoQze+Pb3Ydjt4erFl2VzL104PypTskNndzsvhUmKbBvVeFCYAwCIsNds9Wtp0akHPv3HCZvEcbEikRF2wj5odjeAjlGHP8XGpto5SOFkyrCYBiDqFUcbSfKVMTMzoZN6vM5bu+s1xQnWYJZlwjfedieuXFkSAZF9vtge+g1vfosQNMba8fCbW1u4dO78qLOhjd+gzXhZZskmWlThcC69gI4cPOLyjCgsRy0RN36dkn3m8UYyJeLqEOZY9N1FlTfgHrlpDyvCsMZ4pC7TQXvj13Nn97B66ava0ctXlrxvmrFr4npxX9G8YiMyeRKaw9GeCNMsNIOyfqbKE6Q+88n/mZi63T2OgWzQkPgIAeiI6Wxt503HJNruND0tD9CPNLJF9ERJADY6dshaPlscGWrcvGe1+VANOFROdN0Nt+DKlcsiGjJe5K3uuvtNKp9ts10jGZnDIXY2t7C0tKTF3t0NnJTdHSV17tWRHKfxvmynh1Dy93TqZA+9twq/l9fL8NLHGyf0CGuIvqD+jCYg9j9UXYAsdhSym0hWtaQzeP1b3y2zd/XCS3LKrl694nQwW2gzpbsHxIiE4EWAHOO42tZ9RjlFrzVztFBj/cw//BFnWotkDEmLcUOiaHPU6DVtao7F+uqsMmYDxxeetczRRYg2kLHsru0O6lOoNNMXcRC7YlI/gJ1O2613vh6XLp5XcbmOccxkcdfdb7Z+afXaCPAgAHLxwsXRafajSXK0xjQNPK7AAAAgAElEQVSvh0puasxb9zg7doUgVMMR5Pw4SCP8OfBvPytr5MCS+KB22t5wncczSSgClTQCR+z8kXBwsQG84b73Soiunrf4+tKli6MTl0zQrKCB9xcnnKiemxRGH6G2Y6FDsEJj8hoSCP578B8/nNhxjP7gzh6hNx8XEgDiKpHzF2dHMakfGoEDVmd890AD4YrEF+fT4j+2prSzSEjmkzepigqj5cSk5PMl3HT6Nly8eAbNWl0IGXfg9TfdgcpkVa24wtPk37mzFYo4C3bX8x1pcn0TDiHVdnw+nMj4uxweXyA70NVACk+YasxU9zIjDIc8XtdZ2wolY0fSNHT8aAr7tKAdJX2ETeL1971P110+94IW++LF82aHw79RGOzZRvWIsYPkLTHz2ub7Sj2PHEKzmnHagFDSz//TR/ycdPPiVJ3IAckxsA5CmhTufH719GE81CiTNLbIeix3vJi14e6WpvAMWZgIo0BZmYyFDLsxOG32DTedxoWLBDi27RhmAi8Ts7jpphuxvbkyMjU8Punc2bPujVvYGBy0sFcGUY6Lnjkv2oVj7SflTwgxtL9FoY5Br6aZI4YOkmOobd4rMoYyYd7VP7xyhXBuhzWSYYJjN9yJ+YUFLJ99XkJx6dIFT8zsEkkS1xaMDKKq1Ha9JX9Cc4+bFX3v8xtRTurBf/qI5mA8WcBBy5UXROdsEpEIqZbd4Pvp8qPdYS6It0o2BIfgCr/GGV0kPASiEzF2TJCpmzghwHb88eMnFFY98MBnMD8zrf7m7V4a3/QvvxU7G1clkRScdqOJJ554VIsklE/OmSNebqujowHllTnvXZ/EBCBsXxAwKBzWsM6OUQqKFT+vfi2+ix3NlyCrSCKQNkcIzY8wGrOcRO+faioshfmD1+DosWuwfJYdKmpYY6gpLWKJFUszO1FEWDjPzbYiC/V1k7Aa0STmdmS7vcFQYA2pLz34vxJzauyhTUpt0qRu2GBdyQlzZlQ3xPeN8dQIpqhk1h0fE9rd3t4SHnVGcI/WVVnYwlDdcX/aTd6/1ezgwsWLytpkSK0Z9lBvDfHP3vcvtLPpuHCR2IjvySfI8DAVqSOYvSWnhMpNk7xgn6jY/fKmvdWlhWzWuzvUfbBrHdUd/T52EcMqdV3gSSd8U2g+PxMkujSquTZbcuq4rOixDmTKU7iLIea5M1psljqNvH47RNPGz8+Lym3FDPaKGF5++2ixw2FmOXAwSCTsX37of8lmW7Yodl4U5zP+cFBE9un/a+vanuuurvM+siXLsrk4zTMdGAghJc0Y22BjoLSZ5rl56kuf+tfkodP/oy+ZydBppkmAkkkoNrbBKdB2aOMB27JsS7Isy/iiy+l8t73XUdEM2JaOfpe9117Xb31LXYzxtLvTwR4pSR9LgEZeVpvIk5QJtIYnSxJVoAiPCgRAGTpVePBnQizc79H2pJ1+/e32zb11xtpsf3n8qF358ss+WSdIVpLteGFyvWrBs9Gx1QzLEJWYoCejJ1QnF0gDa19LpQHqjKhFJoxQa288TyHYI0pGTcI0abtzi+3Ea6+3m1f+pz14uNlu375pG68hOVhPcdqonJo1wXvt0kGTyQ1zlMRifHEtAgP/+MN3kgrhZuGHkB580V4nVu2D1nSxWD8qy8zI1O53tZh/opU2C0nPO2AFfxbJfKjG/Sc8JkA8prHvc+2Vk2dZDHn0OM342+3alSs97MgIKJ7ylAvLCU6uoJuqMgVQalnjmkZYpU2W5jGO3oyI1GY9RamedAnPKBgBlgQAYrQBrquDMNd2JofaqTNvtLWrVwiWYHrYqNVoGBZhzHmukM5OngfohMUh19f+qCAUT57ZynO/+wWRKnFociFCiJ3qRFYLtyAQwOq8k7LtG8fESlBX4QYt2u6nt5kSywXWwpBxCKrTIAeeOEnQjG1VgmeunX7zr1gQQC8TrgPM981ry4ImdfuVCYBKZgw5hC0WsIGLY3oLLbBKrqlmqZ/NiFW/p+RTAh5SWaP6ugaqmwpsu/7tqlfSpTxYmKh+qJ149S0WQkDTvbGx3hEv40gNkASzcp6AoEepYazVuvMe3XYnawc1HrTJCFdU4406pdfZbbRjYdNAUkpt63Pao0T4kvbMueIGFqpBXYstG2SmJicpFFZgrPAAMOq99FyvvfmXpKcAVQe5UnYet6t/RNVoh/9WGFeRMlrsLB7Xx+YJz8AowA9dVTun7iH37Rx6pgNFjQOmS7gV/BHWA3TiVD8Y3j7u1zeIc7vAMgVth3U92E6++jaZHzfvrfNkax9k4uJYZk1xVX6vqGrlPGBf5LDFXPR7JtV7/sN/0TmK+q07ZueAC+1eLv1dthsnAMNJ1K9tUJ5TlXJsaj6nPJ3Zi4C9Vi+YHERsR8hnnLB3rK/TFOfxe6Cu/s53ScRD4va97bb89dV27x7w5KMql7q2RiaBv7Q8g/8aAVdoOODFiU6kqFyT90LSJynwJPoeJUfOjeiD2uwxO2Wp0Y3yReDRo8x55s2ftDsr19rdzVX2d3HsYuaTs4xc0rV9/Sv2L1UwPKfEQLG6BtoEmzf5+KNfWhvY1ibD5FOZE231L3XI/8+Rfjqgh8R0OhlyukAGD3uM6TScqxVbvSdmhJKnV8HERQeGPSyJJvGhaBfCxbz1wlI7eeo1MiHTmWq7beXqdQLzMk1eWkm7O4odKXJhBomotjnAVKatV+jkUIVpSAyPFMbAjqzNkkJNbE2CeY+TyGQAMjoZuqy5W/DEVeAgwufAQjvz5l+3zdvLbXVtpd0Bu7OdUzw7ng8jq6kNSvGoh4LVfyrIWWpVb3YO8uTiuV8RSox4MN7zrPxLavIL6c5E7hoLMsKA2d9KzMffcy4XQkfaSrSpGqCYe8bOzXrII3VL5KYF6e79x+3tH/+EuC1K8nSPNB5Qgdg2fTYmQCpdXrQ96V6lEkVHHDloCWgBYMz43LGHnPGl9ClOTNS3snWKh5FnZ77dzh7Sy2Ql3tPAG8wCwbVFSARPQA4UNvPlk2fb1vptjuVYX7vFe0k51CaMsgeZQNBDMK19F+p9Cgx97TzhF8//2o19Q8fFfZcS1qnqm20Ok3SI7BcQCcDYJHrDO2itfaiGOzaGuz2ocJbgaSAAsy+pxj1+z2kSXH9j61F78y9+3DZuL8s32ttt6+vrbR1jLayZ9LzJHThvwFh40Fv2iCK8KHZ8sAEsBvnm2EBQhuTa+X719mkryc6gUcbpfcv6wCuI40n8gEGIWOOXT73RtlZvtdXby+3uxpr6203Bid8H71miADwLINQcBxFHLQ0Y2WQntKANuHbOo0w+Pvcr48a1oYq2ZSP6ifZb4nvzC0JW5gTq1CTcGDavxsg4DVBlcsaCWvUm2rusmiD935BUeLOS2O5Cte2duXbi1TNtA6dgD1TVjQD61bVbXaYZYbg2YQnqJ7UKKN5JVJcgBhCsadaxlKgpdBTIQYKZcq4SStKOEh/6AbbjIBzQ9TAZQAT5aYHSlaft+6+cbvfvrLW1G1fbPYApe11cCS4Wh+y0Yj16+jNxvN86BzJ/ZjGgzum/fPrJ+/TGe87XKiRqNb8QFYV226ouqtrdpz1mBCI2T+p1oCFHBDAECCafaUerUiRzmFjh3E7QcB1qr5w63TbXV0lnhc1GVeyOwxY9B3qzTBvhWLg/X46odsZwXyWElFoc5EGs1ZcCDXVdSrbOlxPznjCOZV4lQsgOYZydfADhzxi5USUJRPjD195o32zcabevf9XubK5zs3ELMkfVAbR+NojIE08cJeKOJU+/x7etP01BiAAvXvgNN5ujkKIyi0cH0Bq+hG5UjRpf8H2wAbFR+3PN/Ey3s2Mel2J6PVbCL17fTkw2qsezOiszNeLJ3lw7ceYNOmRomwEVFurda+urM2FXMnYUqHjLAe7vW5nkxvPtekq0L9Ze7DEDoTxoLsBtLt61aB8mobxW1G5GfDLxEu44ok1R25cX/4MfneD1bl77st0hnQgcOCFMD3pONvYmpLYH5kWwHy2SZ0a/WOJ/ijsPixIstNkXzv96mrSe0p0eG8GN1WXYQOAZzIEWIc/dL+i71RM/CgujlDjgsb6uM3bJPwe5mQpVct2Kaw2AJHFKa6+cPkuqRoyMPAjH78GDtrJyvTtMqqPbZsXw+zlzOpMAyp8Jl7KIPZal0+I0qHMC1BzklgFJkNPNwIQDaMdcuzppoImY2vSJls4ZAEccoOdefJk+wvWv/ov1akQ2nLyEWjbsL4afu0NEiS3BrWhanOaWMI5iiEJJ5eO7N/7Jxfd6R8jMD913NfqmZgvwcLoYI6ePiDnzCnbDyRWqcn96tGqB5Md1kmvHpU5zCHPTXMeOyvmF9uLLJ4hU2drc4MlGFm7l5o2OF0tdW0I3SADY2xVOb6NjcjK6SQkg0smLaAVqtzQxWoDU8eFChVU5N3TG+ZTDJg2pJoqOI2tz7cixYxza9tX//ne7ufw1JxbSbNmHSpIIDpmG2TSSDsATUIg6Uqj0j+LQGrZMDBCe8dNL70+hluSAqBdbR9Y+kRMgWNioA0gKOwVdyYEdQsNfWlajgns4ZUjTQFoWtegFzKbIRimRoahN4Q2+xEwoTTO/+FT7/kvfaxvra+yUQBsQ+LWHRrFtdMIoaVTxgkeQMJoYU4+GY1nbd6qmx6IKqKiig/B64z26AHf1OTQaPoj2KHGrylZn+Pt0Z9ouf/FF+5uf/rTduHalXfz9b9t3jj3J+QfJjDG9y5aoxmgGIEgWeTxsjvjBRDhss7b/Yx9BDt+0Tf5w+QPS1ygLlLgl+12a9N0JghoqnAJwimUze2xpG8GUnoefiUZaeCxtYkIi60Z6uqlj25O1vOm6Dv8ywdaFvftb2+21s2fb2q3raqnZ2WnLN67xwYW8CdiwJhZ1/yAyldQaoEQKMdWkCzelb6tv/AgKVE0y5EfCaEfSCy7BVP9XNXFxqOqTra7ebh988G/t5PGX2xLYEiDkOLEGIdAEGlARcGgQrorHkdUDH5oig9Tgtd6mOMPJ5oPkQlalLKCzJQeDxlE8iJ2NLRinI7ZbiyeV5nRy/xMbqhYVLXYqO/SwS3IAzxLkClUZF1D57uScITo725N2/NSr7fbNa4T34HpQ4xAOaJioZIQq1AxpKS7v5yBToQz5VTCkVJuTtJqyqCqQpA5dHUuxUth/KSldLHFKwqoejnC2JksYpcB32d0207JnDXAtlQxi+AZ1jfEW2zucQwZoFt6LnSPBCYDwxxXL6lDOL5joCKFXjZmT1sTi4SEB36WtsXTizxj8bEZ+P6FSTz06hNCNh6qUDRd0SDEkXtQUlS6Q8HeceZMwZdYXBEA/Ovn6W+3m8lVgSLlRt26taHE8CObbMoI5BTFVaEmqz68WWzk2KnP63YkBB4/aYqfPBOYMX0ySlNJjDVsxIE8lysIeGJw8b6TcNZJO0n6D37xGBLTNHALPxXArspklQDO2s0NOuHtb95iKZqOCexnhXzFE+8OnH/Bk9w2HNDlbJVumJvpsthIk+jyrRQnF0ozmPHPQL0mpjkoQZosM1TnrIOhfeDC8PPovgi6hSvToIjiNsIEnz7xF/jEAnHEfqPEsdGL5qPP4EdFYET5ojapOa7go10WFGt6fm6PWpkQuNDJOzECFIudO79ydKGSz8xcFLSFpcQiUANq24zjajqMxs+manKCnjXCR/RkEufb6EYKCkpSQMnKrqYjDeWXZbJbnAhEuD8JeLmdw6oZn07PxgiHLaWHzuGdcRp0GKEBuEoP60BbcwwID6HU9WbugJ9FZwhAE6plqEz+bbz9CL9gaxkI+pucKB024OYdp6QFmbV5NinjAePhpeNMzJKmihnvNDpFGUZSQaESCykDHTfrcLJxId7pogfU93Pewiz5xDHNAcmDI6eJ5nMPZt0BZ02WdsjXSXhJysTS5X85FFDhyqk62Ptpicuniu+JUsXwn5qZnTika5bO8XCQuajwbSu1g+yhbaT0SRKUXVQkUdW0yBjX0iPAbniAFD5wGCRI3jIYKRNdcIWgP+sGfnyAPORiI8LV8Q0R1GuCq6hKEjjPLYJON6aID4znaCZ34bwq7bDcWcjbRkky6kiEJtxiuWhBjfxlaudFR3Z9qicY6UXNgpMbhxe608eCkJ67jzmd5YeL8cfMOmDQXc1p69+hen9pbBQN/R6jKwfCXPv5N3qKoKpXWuHnGnOUEx7mQsyUvOw5RVB3SfLAb8sQ1mTYmS6xC4u5OD1QnZvP1gv4Erhz8pVWNcnQkVOP0QHvm+Re4qWBTwtfNWyukn6A3ySxWAAvyVtP7VHFawZlhpHIydTpxo5iT5E5MQ9VG4CvXe48qm0yiT5WRPemw7KwUtuOBQDEK4LFOAqn4OEVtx9xWf6mPniZ0GcIoAYxGpq2HULDEabWU2LFWpTicmV8KnZhata2m09BbXUZlDJ/FaKI0ApL7k4wOJTwxL3naUxcwjQf5ZJ9u3BEErBpBLCRIQiqGRm2+PfEn323PPvccqSTxhRInrscMAMD729tkG8LG0dPmu3gRDaiP/dVwtREbd3SttRP+LSEbBQ8+OzabuYKR/lVUEpNh6k5DruCvJFNY07Cxw0Go5ARjU+P9x//JhufgAcwoBy5Jd534oZm0T5MLH/0rq1483oVdIBs/c+xl2fqm8WYHNMwktQWcZHCNcpSEpYs5Yo5zkMqW4GhhUapDe5EqOQbtO5QJCyEhSsjWOXTDS2AMIRrjTp89S55OfA+c33BQOILJbI1KWcqRxL2hbSKgSiIp0zcSOXIKs8AAEEbFwjT1EK33sMthGrWV8W69JOq05nAexeeuTXOiaF9KF9eMNoWwc/18GPJs+TlOblXz6XaJj9A10acX3p0KYTEQFUmu0AmxPY8nrGFPQwTojZY4mZOBZtKecnIY6/qUZL7IiKPtnTvMgfCgiiU7rWIB1ZDVssp9ILcDWO9UW13RlN6Nu6tkEEJ2j+zDYPhzxSxISy2iMk4anrrN7s2kN9PrhQWiEBotk/KmzMFgYooDV52umLeo/ZiebDYrab16WMD9xdPucbK/V0NevAM2P/kJYO/w/ELhylzVCCsagDabF+bpHl2JSONFv4v1aFRRdDId4xkpCjyV0psD6Ie/0zFQykhT64o9g4MWPDeegW4ZhrK5vpzSphZ+FDUEPFTv2Cuvnmkr167y5e5uronczYkdqjE3K8ZZVNyMcBJOHGrSek+ke/GFgkpMC+7BU4TnOuAikWktYeOl9r35hjhp2BycOxs/x+3MetnJ1MFBfludKTBP7Et3eKf9MG0XES0DRcRN5vQDHM5RtIr2JC22U8JB4cSBnpz78JeKswtTLz3yvZEZktrTw0hy8AAOLQy3ibSl8Wx42cp88TTCMwTkx4uEFRmqBpkSXR+4NQmF79VhROJbSYQA7rXjp063G1e/5qJt3d8gYgVCxdKsNUV6oiPhym0btEBEKhZdqBipSxHQJ2rgOAr3VGX+p5Aoo3Ajpw68brovpBFrgPdmehmzxgszFKpcMS34LBNYKSfjul1/SqBSWuY77Gl2N67fSXNc3NFUxZiWcXhpsy9+/B6LnWH94xksqqOnMp33jqOGFB4+BqaeWdugGVgKbVBnvt+WOO9aJzfM/iwPTveYhMClU8+G972I4kSHEkNbiJlQEjq0x/bOtJ0+c7bdurHMzQH98vr6Gm12TwyRqQnZJRHEQjUne8dqUkh7Jgca5lknjGKumc6oHDe0KjOGR1vSA00TTn93PO+0HkOYMVtLGyikqPyA0e0Slatr6oTCvMmpVVwvhKlgVPiKiYRgwy/Suks4a7TUEy5WL9xoCEnd7NjQ/FCGXW4lZAWSGbUGT5eDUuz49MDeN8DpTBtwVEzKopmDOUhwR4GCqp+w370+sD2AgIAIEepx8+cW2osv/Vm7uyZ2QHCRX7++zDHInNG5s026aPGaisRWeX45atgcYsvIqCBHM0PQsanyDVwx8nShhGVDaOVgIfqginU+H825+uwBhoP4PLBkAQlkrSEQ2fCUhKN2c/BynWQy8X1om5rBjOfdVbYrez22Z+jFk63TkpvGkajA9rSuYlIffh7JlIqEIKiYEs8RN+8xcWcDVp4Ym4CXxwMDyYm5GrhGkitwsLiAbmLTiXHNuKMolZR55pnnid7cxcjG7Yft9q1bYmBIWLgLFWlqjU5eo9HJQXsQLmQikRAJcBNcIOEkQA+HBSgCwgh4b4bajd5ybW6yWlgLCCiETHkJYMWlIdI8iaQLGvmjqnFtrgNO9UzBTodOZkbTCuTfKIGEZ4BpwM+zrvHQuwBks2OL8+ewJw6H7IFCF3Ni3WGoZn2JamR4h5HIJF6wcHHgEo7lMwT68T/E0wovSKVpcLwkVlkraJP8nDXi6bQdXnq6PX3saRK9ovEdDhoHssGjNEpDmkWxKE6HpuSJ7opwXla0RPADqUtrUJxJOnT22IMQSVO9FlKsSAk3Ewfn5NHj3xZB3UxBCNqyF5ZS6gUEWQPl2CJtxAvuo9hfMXRYDpPLx/tRU1mYoE0gBKHepM934fy7PY5KPJYTJifdRZJCCSkPO2KnP6v6CF1HBCcaItAibeDwvOvvihpT6UyoRhVCNB4i92WSBO2rjx+3g4eOtGf/9Fm2Au3ubLfVdbQEyfFDEoV14eku2RHiiCoxInADrquKuatXCBMJbHQPd6g4IVydiK5kt6zm5YXvtsXDmlVK/8CtuVgH2VRdm3l+1w5U+VPuQRnFsZZsP8JweAsl1gyjkbG+bFAwVGvUuZXNSddJNDQTM0hqZbOTcYlKr3ajH+GGmRaa5BrpRYkwdk1ORkhsArcdUJ44cvlcEgVJFQZUgJ9jQznv2qMaBpOCFTrGP8LxObjQXnjuhba6uiLmgqt/5IJT4OLFp5l9H/BwRssYANE99vCrOvkD3nD9TJtBzWGzpbDQwm+kT0LKqNfkGhA2xbGSI6vWXmUItykETASlrm6wJwWyx+HGFITN2Y2QMHS91h60ivMkPGBffPbvU0gWbqzyn9R0Xjqbig2A5xwg/0gc2GlzrjdqpSaEEuPGS8y196dgByugVGPgSLGjSSRQLbtmjVLn8eMnCDaEqn3n5//UfvjS8/LaCb5YEG2XB7+HmUGU13a+vE9Y8NFtOcq+FE6nP4n/DkOzt5hajuXLAtLs3RwqCPW0rFOyma3dq2k6QqpVu7ukE81mMJo1BIkPWKNSviH7ldw6NWlICwsMmg5aJDXNbPhw3H1me6aN9ihtMREAOQAmijfAQGHUKEAkNSoEptCQ+BPCFQdCp1d4ctko3XMmGgj0Ju01ZleEnf/nd95pZ86cbv/4Dz9rf/93f9sWD8+3xUOLnB8GbxueNuNSsCog/jVlCEMbb3TQKR0IWPq7uA1u8Y0GDL02n7Hi0p0jTZMFO1fpvLoNyZzobAVWQbiXJ5N3p6oHHYjbh2nWDJcCQzPeGeu4uLRkLZsSrBy43vi/73RPLl14b1pZimJ/ZZMVf2MjOLBlH8mNPlP6hVPJ8bG+u3G3PfX0U7LplHrFhUlyKMQTLzgkP6paDs8YDRmTEuHA1VSSVC/1Y87sRBPhw3ZwihLnNz7JiIkftKUlTNgB7xlCL/V7YeKuSAKM9nSbrwo26ekOl5uydez88OmjlvJ7xjbG58m/eZ0219bW1zgkhtqFhRiphK6u4/OUHEc1p3aKmJRK0Yoh3aNHjCggvNG0iumFQuUhKpypk0sX3p9ubm4yoTCcrlrBksUeIL0JHSV41wn6ZcNjmwPzGaBD2ShVYSCRrF512g6hNdNWo8+FL3WEY0m8xF/garFeiGQDxiIjiy3BTCZqfjIhXgsoEKxv4lRQXfPkmesFz/fNN1vMpYcbpfssLKjITmcqQA6CwBpKM6eDJQjcVEa6s1vmqGSjKRRutpDGEeZOTJFpNRoeU54pthtTgZL8GTBuJ19szyM0vBc2OxL57U6ZbiZ77hFNpeEbkqVwJCeieucSfgLj+u8rohWFpuJu5ZI9ycBCoSyXwQ8u0EcYR5Sga89hlBHnj+gLagxOk3LvimnxBRN3//5WO3xoUaB7xPHz8+3QPOLgbaVQd7XoOAAYldSnHIw17/6M1kOFHsKDwEQcjHotItG+ptgj4j/AhHDqMMeD/kkn1TPmb6YWoG5PxuNYN8dPoAUPlmCsDZ5JPDShCoFJo4N2+ZPf9s3GpmdTojKrg5bNrp57PNrYOth2Zc6GdqAtBidocN8Zv5S5GS44xGEj1bJDF9zTfaSdB1Q+geJ7OVomk7U9xKhGxZdqm03SvWYI8bzppWIee6IRj/MW3m67HSaBxTDpzhyO8RwqicYBlUPmvHRYD0ImaEh2h3V11gph/ygwKI6Y3A4nPp8VocCgueRmylPrzA7adIV9cFjjNPJk/8fl302JPCzzr5SEGHTGRajlWboPORs9q/5lnxlzLqonKaceJy1pPZ40Oyg1BOLfozatQUgQU8hsc7+Mn8pmRwPd37rfjhw9qkEpHuGgbNkA62Xj6Yi6GY+x+67CIWwe1b5LuECSJgYGGPLOnY127Nix/2f6IgjQz2n4i9qWdhnVO4aedvwQdiE7FzPFOFzODu8xYGI2qRMBMzmG8cA8w9T8Lip5iXhkFg4wvp98eumDGXxCbHNOeAXwRwhy2hmse2J8atjZCHnYvU6mGZmeZ8Eih73zOEP99+yJ8h7FAcLCQ+UlYpAfIMHqwuZ5liNe1/35Lv4c1X3meblJT8+g08HMFNbYyBPlx3MPwZ8hCIFSJSunRFBoJvX5/VqxC2k89jIlKbZ1HAZBmxSDay112jXgHZ+7t7nJwg5VPFuD9sQV68YFnHx8v5c6ocbjIWsBRzEdL5qXIpDPbSfDSYqNnG2pqfYDf8c1qhbQQBi03oxMnDzYQTyjQHH4CBRyjDGiFtImI5SS1BvAaK4xLBJ6v2BSxvuMal7i+TwTFjNdILDdMDlhJkz7boQ6WMpJKI8AAAdhSURBVHeFTPM9/Rqn7SGm2TLZokWOZ87nJ3wJFTxtWl2TCMY4SHD8nO9wf7g6QhVbU70/gokKBbj8VZk1NxaWfAk1xOXLv5/SPhtaEw6x2G+l8gZTQiQvdrtWYvAgyYpF3UeAcpry0hEYwXoH9kzJj9mxilGfta0X8SbOrainFL5xRkhaVL0IQbf0Re8/l6DqkMlOjAVPn5g1aY+5NQmIGss4M5qJEPO5g0MaT8UTrB9ULNYFEUzleckzVXufE571iTnVeqpfLHYYzI442VwXLazv6VYuv2tMwOSzzz7iZsvDEyYq3mtuPLJiY6pMNjvqvnrrWqJxklIQiGpXCJbWnrGxuSayXimPytFTokYxcwowOfXwgBH/Aq9u4rze751JQGFuHAmfoDxiampdOUmdYQORFxdiFT8TJaZBfGFWNudKjbBy7RD+5tBwhBRNgRJSWQtBqPT90cwY7nIsqPP5ps0A4RBKuHpOTQfsozhKQ2OHlGGz8eHqqWbzUz8epzykqFC5QY1kY7Upo+gxWoaG/R/9xFGvtQ5bncR45ji5meKjk5ci/igYxPGSWgRXqVOdTswM4cvfIoiBGAffpsORcIr3Mxl+/02364hFQdGLBFuqM4DGrBlMFd5V5rACE3WvmkmMd5/3UM1cdfZ68GifbVblAMuRC0NEogL+jgs+9Ds+//xc51SpH0p5MKiObE6kKDndqp5rPbyq8bHE+lskOLadoUahg8qmj2sPxCfGIIhZUClQePxaCBPjwvbbYQmNNq6TGrJSkE7d+lQmWRLnbzhW0tUiBxi5+pz4qn6x2XHWlMMPBNgJmd4TDm4ZIV5qwTo2/969LQpGZ2xy/h73TBkzZgIags7XnCpd1T/oG02NZ8QrNjtSk1NWN50pOvdJMzXKAWUhtk0hAY1pGBAumqmqKbJww2kbZdMqEJHq2PiYAZkQJVeGV6xTgRQu0SX2/BGC4GVUsx5hTH+GjGvEe6BZgfPHFCb2cMvJnzwP/qQ69vgFePO5djZoqOtBWJDTCUEJiie16W9zziJAua+c2j2GeEAE6T2Vas7BgBMatNDsgTKYz45sYvfJF1+cFw9anddRSlYjoaHm+AhGbJaVeMc/V6ejhh9V6rT4aQ0a6jhCNpw6lDrdb+wifjYuzxsBVSZPSQdWoAwqYJxpZ4mkcalU5cSYKuvBw4fUEuRutIOVEI4LzchE+Paoea/GjI8Th2q/TzLUveJkkcQP9RxBzmZn8/P9CBQg1keOLLloFKbkUaHTvjjTZh5Xric88//8XDZbLrw+GDWkgsUgcmNhxMWOvExV9yqciAqK0GSX2YT+UP6bed2OIEHixm1GrhvHo8c1hkerNtZasKnhHTZDi2xwIBGv0DI6BQinDh9eGsCA7n8Hj65wCM+IpEo2O2iQnETew5oDahYLOBoAM21wIGarxqwaLhmxmouoMbjWAKp+ND5mPaJpIgSgBHvyyaOMtSHJ/YAZCxw7zh1WnA0vT433mT2ZBIqw0XoBVprc+hNtkOZb/Vt56H5Dj3msKoZ22JmsEepI3qr5iGceCR8/F2xoVqWbu6yGHkUooRJRi0fOLoBJBR8WPlflWBErPK54huQa8g7yA8yYmNGI1hJxxMhs6CRLTqScqoH/jg+E90h0UgWY4bCLRtV5zufzp1S6+VFNeAAPPbTfSSbxmZFBq55xJEc4LcGH5GVrI0EAQ8fEpzbSmbId1zDcV2bQtVfWwQL5d+gngCiJk7V/w7UnmQ44xk50zeLwUvH0MDNYhEMkiEOodJA0mouHl8hJokze6GGTf+DZIrPGr2cBq9kQkFBCzejezmWEPJue39H1k6cfEYUEwKEVhxBopHUEJEIg1a4GSp1wMSly0KyjBX7fh4BTfQEgdXMh9hICMJMujWRp4VVPjuufF+nqPjXYzgIgz5WntcTY+G74TmP0qTWcqWMt24akdk7GpkvCR9twTnwWJPY/mw2nJeqf82bNTMgcOMuhYBnU6GcszsEF0UzVzc6192ukaBeZORMRWJtFSCMEw2fQy+XfEhTXsn0N2nN7/DtZF/8shy+Ck/tqr9CSrGIINS8STNCsPjwo+vJQhEwAanxspLzrYMJif+Nc4PuCz6rmTKkMrpr5ZJUsuTlWCTOJd6vW1H5xX5QZM1YqKjtOVcITLeAgxgkvSxy54cmbiNbsDTwnlPgQ9nlSoPlX8axy2NCgGF6xkf2iBpvF8/YTHRUPXtCcQDx3nLrYeTbulRFMSHAwDGQXrUqwOKXEoO3stKWjRzsQQSHfWMH8HUxK7D1zFm/A39y9KenyaGlV3Kmlocbria6OQiS7OkuxPbKD8F71QJ1+0r9E25yGP6u8uvFU/24zDYlrdVjiE6g47+S+a+PDdAxgdU5U7CliWXB2Yqgc4LoLwHujros6d6V4dmGB7feO1SNssPOY5Y2vsXnjpPJeU+H3EhYpATL4YhB/R4j7oeImSVvBK4eNX1wQ5psACg+hjQboPlCiJm72nAbYl0oe7TS+7/73fRjI9n85OQ8T7wFtAwAAAABJRU5ErkJggg==">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -795,7 +852,13 @@
     <xdr:ext cx="304800" cy="304800"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="20" name="AutoShape 14" descr="data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAHsAAACkCAYAAAC3r1GFAAAgAElEQVR4Xmy9B5Sl2VUe+t0c6t7KVZ3TdPfM9ISePIqDRhqhZAn8DMu8hXnPmGXAawHCZDDmwUMYk0GABcY2wQSBSBaSQBKDNJpRGk3OQTOdu7q6ctXN8X/r+/bet+7o+fbqVene/z//Ofvs8O1v75P6ylfuTwaDATKZHDKZDIbDIdLpNHK5HJIkQSqVQqFQ0Fe++Du+n7/j116vh1KppM91u11kUmn0ul1ks1lUqlV0Ox19bjAcYjgcAAkwTPi9XYfXKxaLun7cm+/n/XuDvq7fbbfR6/X1Pl4jneZYEiCd1ec5Xv7ni9eIMfIavC7vw1fcg99zrNlMBvVaDYP+ABOVCjqdDiYnJ7G+vo7+cICpqSmUy2Vdj/95bSRpNJoN/Y3XHQx6+prLZFGv11CpVHQvpNN6P+eB9+X99Cz+lXPG8fErr93v9/X+mAP+rt1u6/7xe36en4n38JHHfx4MbL1qtZq+JgO7ZjabQbFYQurRRz+TJACyvtgcDC/A/5zAmKj4ykXW4g046fZ3CklMLNcAyVDvyWSymkDekO/JZCgIPc46uFx68H6fP6JSqaLZbCCTztjkcuFgg09RQAYDDJNE10mlbHIyubx+jjHwPrwff8eJiYnm2PL5/GjSY3K5yFxwjovCx89SkPj+drercU9MTIwm2+YgrbEUikXdo9Np6bq9Dt8/0PizuSz6w+FIiDlPMU6TBKDVauna/Bs/z+cZF8zYWHr+VErvp4A1Gg1sbW3pd5VK2TadhDBBqWRj5TU5tkzKNif/a30eeeSzCW9EqaBUhzRmMiaNsWt5gZAwDoSf4QXGX3wgTjDfpwE2GppkLn08kIQ+AbLSHKYN4sFarbYmm/fkq8MBZzJoN1vo8/tsVg+RzmYwMzOja8YYOAl8qPHdHRPJa8Ru5vslKJkMEkp9xrQDBW44sPFo0pEaCXOz0USn28G+ffuktXRPLnCvp89QSMoTpp14T16f8xC7lb/jz3x/aAj+HEKgsQ+GWshWp439+/ePtGyMnfcZ9Hsab284sE3A3ZskyOZMI+dzuxsxFlnP0uuaUHGxbQdkkMvGg6eQplhwx2ezI9XDwYeKp3qhpPPv8Qq1rxtQLfUHSHH3+04P6YWEwXYIP8Ndwr/x//b2ttTOxEQF2byZEk5Es9mUFOt+aVPNMRG8X71eH/0cE8txUfXHK8yGFjpJkKdK5GK128hkM0hzTLwfhaBQ1L34GalvQIuhuTIjos/SJHXaHZTKBY2fgspdSIEYN4tUrRT8MIn8Wwidmb8U2u0OUukU8oXCyByFidI4+n3kc3kMYLs1TClNCe/ZbpugmrkbjjZNMZ8zIX7mmYcT7hqqU74K+bzZwIxJTbw4UP6ev6OEUgVJsoecexOOUCGyYbk8qKz5no3NdQ2CExFmQjug29X1ymWqnwES3xm0vnpwV/cxCqp1jqPX7vBxkc3nJQSctGq1OhrruI2L3c3J54Rwgig81CBSdy5wOZoPJBgkplI5YVxYCdtwiKYvYJg3PsfOzo7uqUV0/6DdbWsecrmChIjCzvmlLdd8pmyhzBylpJK5cfjM3ADtTlv+QzzDxsbGSHiq5Qn9jf7EuGngfIdW4XxwLkJ1x9+kbb/ylQeSMp0E38X8pe1YU9vhjPHBeSHZJ19sk54JORJUg8WiSbfZNu6+oSai26V6tuuFitNuGZrTw50sByudNtua0KY1sb21je2dHZSKRRw6dAirG+taBNpH2ihKeKjDuG44llxYTmjsjBi33i/NQ7tb0PWnJie1O+kzFMsVrK+tI1/IY35+fuRvxFyMa69mo4Ecn6/T0Rj17IlNfKfTs53X72sjcY6pwQqFnNQ+BWVlZUXjp/ks5vJaAy4kf8c55e/54nzKbGbMNNCMhXaKv8VGDBPKcfLznA9qPdnsxx57KOGH292+VEkpbxKdSnEf8UY2aDpwox3mNjkmOLzyojsLcsiovodDPSQH1u31sLW5qZv2B2aLudgUECrJGKQW39XpoD+UWjOv1zx/Si2FiLuF+jSdzqDb77k3PpQnigGwuGcR9Tq95kk5W/Ja+wOZjjTv7d5uJksHic5kHu1WC8ikJQx93y0lqdTE7pGixkvrs7LJYcYonM0mVldXUCwUtfuSlO14037uZfNGqZTsLn0AzpG0B4Bex7QOhY8CxMXms/Kz1CKT1arMDl+r6+t6Xr4nbDMFM3yEiFBC8MOZTj355BcTqhpkslJFGdDB4ETa0vZ6HQ2aaom2iu/lhHJgfJBQY1IX3M30SD2Ei5Aq7DE93xAgqTEP7ai+5Xi5d08JplXs9xP5EXxY7cApk9R+zx2gQR/JMNEC8R5JYiGWpCexHVEsFTHw8IxmI5fNabHtfnwiap8ChoNEO3B9Y10LMj83p5+7rbZMVofOkdtwOUU+rjATw56ZQfkrFNi8LUy300V/0Nd9ad/Hwz9+Nmx4q1GX2s8Vzcni83CMVPGcf96v1WhKC4bDG+8L7ztsdcyjaVWLKjS2Z198IqFNkgT1uihkcpK8YWKhQKgLTjofIn7mLih76KAwhwvsNl5T6HFpSLWkjB6jS608U9nOtNSSpLvXe02IRBulsML/ZuaFXrTZPE6IHoKeJr33rsX0nFhei3aWO4LPxWeKUIy7k2q81W5pJ4a3TO3DBdGOTZuqDDVqiwp0JVR2fwvV0nouhYa01VzU4RCFcmm0q/nMNCvhryhUpUD7HAlTGPakbrm4IQAjjZBOj6KWcDLNL8iNsIoILWOueL/Qlvydnv2p5x4RqFIulc1uwzzbcqkgCTdny8IVOSeuiqhCQqJ4oXBcQm3JexwMMOngQ3jo3FUCWuiM0V9JpxRiUUVxYSOc4PWnJyfNi4Q5TXpQJCjkC/LaeX8+JD1pxrdcKKp4TmIsFEO8drulxZVJoK2mk0YB6nYNtODOd+eQO1iefio9MkXUAAp5ej20uh19nhM5HkoVsjkJlRwlmqGUCW84TvGZiGBoMrtde26Fn7Is5vxyTOHAUaD47KGyuXBzc3OvCWUjnAuVH+qb742/6XpPP/eogkw5LcMBCrk8mrU6si6hqbQF5IWCxb5STZykUsnCKk4Mna9koAGN7ARBAvfeIzzjoLk4dPT4PqpIDmK7XhvFvfzM7MwMWu32KKzLc6L7nDhDybiLqRppTkpFQ6K0A4e07ebwaVe4g8j7Npst/Z0mioJRqVb0lYLNC3KHc2KlGt1eT9BLdmSO9+ecMIwUltDrax6klRJaDQN6KMC8Hk0HJYoCxleYNOogaaFOR5+nNy6zZ2/D/PzsSKOG4JvDa6/xWJ6fD78gMA5uAqGh6YzubethplWLzZ2hsCABOq02qpWKSSehR/q83ClpAwG4GNyx3DGx66QmcqZqAjyhMNTq9dd486PY1uFBugU0B4VSUXZ0HC0at4+h8kIoQ7VucXfT4XEAQ0JZNGiXoZs8dtdMXCyzm4kBNPTUM1TBpgWIehEmrUwY3KmFpOYo5PUzr5dn3I+UaRIHXei48aXQldfu9qShKFjTMzOjiGZkN31M1BS8PwEbLUqhgEa9gYmKhad8hWoObcnn5FgVkfR6Ei5uHL4/5t6wCEMWBU7Rdxmak5h66tnHkoBAOVmUODpOmXQKDC3MVqX1gFT18pZztDe2k/h3gg0UgMCF+X6qND68QhXChfLOzRSYM2UOoL6nL0CwJLHYnrY2Yn/6CozZOdGESTWRdK40Jj68LZjtPBfIlMW2HCvtOHetoNax8E82t0sVaVJvCF0GRPEYslBI+FwMnbhr+ZwUBMW57plzgTkHfF5BpA558rliXqYqVY2NWobCymcNDcdn1Wd890tTMqZniOvQzfT0tASJG5DzEoJuzrAJGsdvttxQtRBwrolpV4tkUi+8/IwjaLsgCgdEEF0OBBfL1Qe9VvNg9QtHwMzrJfTJRaEKlQfoi0nEZ2NzwxElG8y41MbgLTGRlwoM3Jzf2QLaAyREy2lfAallhm2cVH7WJm4gf0A+RD6vhSKerJ3q3jd3KLUBF1DXSlnSRzsjbQ6p7bAKehJYe1ZeK9RqxNpyHtMGJnEX8sXvhTJms2hw0YQZ0GegYAwVj4dQclEnpyYtOeTTyvFwiiLMpRAqWnL7G5uEfku9sTNyOu3vKdn78MCZhyBIQ8xEavyZF59OtIiZFPIZokwNvbndaqBcKGEw6KPoWLW8c0mK2Sg+kOBFd3CUpZmYGDkFFBpqCmZcwqYp5u6YrZH5cODGMjp5CY2841xOmoVj4TWofQK14wSGdqA24WfDWYoIIkIcU30ptDud0b1kagbEx7N6BoEghCzTad2Ln+H9+BniCwZYDLBTq7lQM2IxRDGik1TWsk0Ubl6bfoZ2snvcMZ4AP8zh7KM6NWXJIvoXBT4/zUxfmkJ+1MCwBjqTvP7U9PTImTREzoQtwmD+bmS6uhQUcxilgV4++5KEiCBARmrUEBxmcxT0p2jPbUcRXOC2swU39IuCwt9x0gjtlcplhWHh2PDGdQL8zaYGPlGZ0OcD2aIzxJ/lpPCaA3P0qpOTI7+B15eEc9CDvsKi8GojpjR1Y1omJpYIFe0bNUCn05ZfEF5xqG6ZBU9cUBtQi0i1e+aI9k8qME3YNJGGKJWKSIa2kLy/wKVCVosRjlK/w4wefYMsCDYF3Mz3M2oggra1tY2Oe/Czs7MygxGXB6bPZxF27iqeP0sQ220JFneurunp1LDdYSIVy1PLyWY//1TCC+RyWYM23bGhyrTQimogh/Qw0c7iwwp6c4mykMrsnh6eNtRVeG1nR6B+2DA+CCVND5LQqelJYmWvlRk1eJYf53hGgMWQKnoXiTJNZHlzLmAAGgrhaNv1ecPCeT8JL737HLFuy3QxxuZX/p2LaGAPowWOlwtroVOnZ37G0L3xiCzCpvO5OW+0n51O10wLkbY0Q7WugKq+A1S6n4dk/IZhF6OOgKQjvOQut8RMSiqcY+dzxqbgnEYoK83nDhqvR/vOr1wzCgId5Ugppx596pEk0Cthub2+FpXOkGDPrCUMUkyMM1HiMabCINlXUyN0lCSBvnDcoRQMOkemWgwjpvetzJDwdMavGUkdFzqIArHLLRwkNErEzAAOLgr/zpBJpoC73L3rVqcjIeHc8p7joQntI69BoRHSlBhAxPHH/ahOI1mTTpl2IronGzow7TaO7UcsbOrUEibUVFqklAMy/S7o4kWem8/ATcB5irCJX/lZjpfzwu8j8rFM3FDzzh0aYaG0WJ+hZl/+CZ+DIhs+Q2g5aVHOMX2OrzzxsBabEs3kAzOblvUpyIYw7JG7z90c6kJwqKl0hWeesjTPkHivQYMCMnyyeE3loxXSEK60XTk+6GBtmP9HreK5Y4kZUKvtaLG1kxxk4b1MJXeVaJAQuoaIxRMY4lkrM0kWr3Lx5StwEvs9MK6mA0cVST/DQk8TLu2uMUcp1HVMrrJ2SSJvXlEKIxJh8gyxnGDhmTV+Vo6TmxXZW0LGLoiBuMnhYx6AGEOwcTx219iYMWQmMaITwsaDwUhg+RwCv3zTpB5+/MsiL5hX20POSQv5vDkuXGzFa2RtkHLjoRQnmw+hz7ojQlvHvSc141SkwMM5cE4Y6UWUQEocU5sUsJBCxdF8KAdPtOMUqlhYRc1gnrQtgMXLWak8MyW0nwNPF+6SLwK8oE2kAIQTQ01C28nPa/cS5iyUNEFcAD53eODhcYd9DHAj7DavG3FxhEImtDaO8C3CxDUaNWmY0A5M1hAj4M90TCm4XGgKJ0OucAYDIg0oVQAPYWeaNUfslDhyUItaMfyY1GNPP+pMFYt9mSDnhxrNuhaYzgWlqpwv6uE5iAjutbPH+Gjc7bSLyiyNATDSAo6XCzcfZc2C/ODok1N0LMzi5Nv1OB6OY2enprw3BaxQKJoal49AEoGBJYwciGLxPZxkqr+AGyNRMA7YRMxLdWjYQErXpSaIxYisGxcu8PtwgGKxKbTB6qGm0AJ4WBhUKQoRx8+IhQIsP4SIH59xLEbnNRk2hRMs6Nk1JXludHjDBNIp5Pt4T3EISH4grE2giBh8Pi9TKij3iWceSyg5TGVyMFnu7I57fz2qtJYgSdocTly+UEK5zLQl1bqF/nzI0A6GsBm5kDtcUF/CHWuYeAAInHCCFoa42a6MGNESFvQwzQwo/CAE6ULEh+N/20H8m/JAcro0CQRcGC83GqOxxU4Nr5XPKgH0JBCvx8WlL6A42Yl9kXjg89GX4c+2aJaIiMWmg8YF4hgopAzBNzc3R7loOYtyuIxXJ6zdSYYUNGooJm20OMp7M09uiKRsuzuIyk0QtMmksbOzbSEI4+uJsogYEcJFXB+OM7GD1Jce/aJsNrHtGj88HEjd5tMJup22EvrJYIB8sYRSqYzSxASq1UmUJ6Y8xKKDYyqf6pA340LRVlG1cuI6XebELbnP0IYTJKTO0Z7AfkfeKBGxXneESAkJC9za0TeaAJoMjr3bY5zqSBi/IoASU9nKjrmpUa7aKVAUXu7+yJ5xYiIk5ELyvzYA05m9rjhoy8vLyGWY5m3ImYpEBdOvBw7st3yBzBnnxeJ2vm9udlZ+TrNFUqUJI22tOZ4MpxjimQOby+cUVnEHVzwCoqqTQJaK0mB8z6WLF0zbFkpm5sjedSda8+Kw68hmf/mxLyX8ZaO+g067jmGvIyZIPmcTORx0iOojRQaGXPoicoUiKlML8gRJdqA0kiJEOHUwNFQqGCfaCV1yy7bk/Fy4cAGLiwvYs2ePecEOH9KeinjgryAdctdzh8euNrtkSX9OEAkKVOMUDl6P/zlew9oTQY8kSWSFtqVQKhSxtramu3CMAUhEJDCeOQo1zK9rq1c02advuwOf/Ohf49a73iCHs9M2XDoyf+F/MKdgmT9T54pcHCfgV+IOnLdxti43bbtlISIXmxrXHEFuImozmxyxiJIEa2uGIzBvwfmi3S+VLWFFTaJMpUgWBqumHvzS5xLyoNu1bQx6bXQb22g2ami36yCLI5fLmFpk4l057RQq1UkgW/IwKytUh7TeoiQsh3K5guGgj1azhYcffhhveet9MgecUE4+NYFiWIVK3EGkPNmDmUNkHjOFicTDRsPIhJxsqubAyvk3OljdbkdmCJ6WLOSpRSioxptmOElSgBZ0OJR65cQyAgmTwPtywng92UDPpIWD1WvXsLm5gTe+5W34o9/7EN7zDd+MhESO7Z0RHsAJDQHu9Q13N66bRR1yNDNmvgwhsx1Oc2eQr+EMNJvUKPSsFW45Pp9JG75BU8DfUROb+bHsXIZhpwSKiaqszKbRr90UfvTjf5Vk0n3UNtfQbzfQbTN+LYgmw1evb+nMtHO4h4yrBZ4QB88jTbJDvojiRAXF4gRKpYoGJL5VviDItdHpeVrTmBOBo9PmcMEIhHCSRdFxZC5if+4+Tg7NQLvbcWpSRfE3QyXa2Ga9qc9ZmJdCtcpkRV8U2vg9J4PcdArG1tamcHZOEjNh/EwQB8JciF3rW4mfbTS2UdvewA03344/+59/gG/51n+jzygJJC/egB7aawpKs1l/zZgsvcp8g6U9RcaUo2lzIoFwX4S7lbtaCaLQViOMwVk5bhKEySeGFWTyTEUXTJspbBsI8qVzq4TLX/zZf0u2tlfRqW9idqqCen1Hu6TXG2gnKF/NZEQkDpwJkmT5YMwDTyBfKiNXKCObLSCdLSKTy6BanRKVaXpyGps7dUPcFN7Q4zfHy0APc3I4mIhZd4n+fVQqEyIMcFE2tjZx9uxZLC0tKQ/Mscnm0oZlcyjm8zh27BiOHz+O6ekZdFpG/Y3EA2Nnzjb9kJ3ajpH0U4aARXjEcZjGsR3HCadz1GzsYGdzDdfdeCv++i/+DN/2r79LGiLoxeMevj1P1xiwYv0MtYvDJ1EWjQkPX/TAsoMsEk5faDja+OAO0P5qw4CgEfPvpEQXjXiS92oRYhTOy6P/QPuukPnDf/rBBANOWBubqysoTzhJYWjlJ5Q8euIcSHjc4chIEDI5qZpMtoBMlra7gHxxQna9Wp3GxOQCElJkCcP6i+GdqjGodpBCd2ATzAdReU82JwDlxZdewksvvYS1jTX9vecxcuzWcOzGVfHoHtz5JUYPBczPzOL06dO44/Y7BOoEZYcLFHbbgKTirsOWSrQjDB2DdnV9Yw2HT1yPhz57P97xvm82E0LOuUyMOUfhW9Cho8Mlm8xQivj5iPtmi8fn5e/DmVVenqZnQAEzDrrSlA6bCqyhqePadNoCkoQRgMCNcpNmNpywqSSVo2rSJb/xKz+eFLLMTfeRY/oysbonVmGYnbGgPC5CO0Q3n1IXjpI8cd0ASOdyUunZXBmV6iwW9h7FEAa+iKtFe0ywwGNvARwYKmy5cPkSnnnmGZw5c0YL0uoZm4NaRQ/ioVKABLHYoeqCIBDhEgkVfHCKFBedCRSmGMnEvOmmm6QFIg7ns0Y+X0BFwsXxWjKyaTZWsbp0Ea+756347D9+Cm++712iRtEfMNNjfLjIm9PTjjy9tJrnlhU1EATSHBAM4WLtEhW5Uw1MIQ/Acp00WSJe+m4NoCSfI9RMoqcnnpwzyKRPVI44XGj3+LX//P0JbVKxVECKnGXmdJkA8cUhmCV97xmeqMXiLjCuuZH7hCwxFOoPMTk5jUw6j/LUDKbnDmFyZlG5XQoMUbrI1jIuZCjz4osv4oXnn8dOoy5HLZIe8mYdirUFNI6a0Qu5YUzqRy/BmYwc7DchFBa3GzrHF8fBsIg7l/7I1NQ0bjx1CqdvuUVJlYjh47r83M72GlYvncPb3/3PcP+n78edb7pXBX6tesMWeWglReZMmXOpHcl/TvlSalh+gKlxIYb8zMDoTBEi8omocZjgiKcbkFYfxZBD80+4QfVMJC24phDsyhwFMQg3vYFmpn7xA9+TCIhPBihmWQJEN9/LdrSjzdBzNxIrV/VleIeUfDkkeaRdBXECaZyZCJia24NuUsSpW+6SNy4MmA816GNlZRVffvQrePXVV9Go1XVN2mYLxQzgtwW1laMW4WLzRS1iEmsPPVLd/n6S+cY/GzYw3isChvLmNE/GvEwPWVxYwVS1iltuuQWnTp0aZfc4ofXaOlYvnsPdb/46vPLyqzh2/U2y2TQtlrbkeI3kwBeflTl5YeacI3rVjoFHrK9lF2c9IyxD8XmAJq6OhRYWC2hRZauuwoTF5sTSzj4tUtkULoOxeyq62N3ZKaR+6QPflyhWywJDJh6YRRrS1hhFKQj7uyGRTbAyQp7jNpaG2fRR2pDFe4UK0vkqbr37rQIWRLYf9PHZBx/AU089iWa9MWJNWrxrFZ0Kl9xWxWLbw9kuEanPvW89rDMzYzEJqkilxxZ3Idjd2TZ2qVenKvNnyzkbIsg5IaBx04034fbbb8fO6hWsLl3AqZtvQa5YRaFcVdIj8TqrkTlIGS1bfgSdUa6E72gOWz7JWHgU8KuhjtSNxgW0/IFlBM2AkZJlSBsdM1HFXJOEuFui1lBN2/l0DFmk6MLxyz/3/oQDK5XzSDn91x6YWbCWFps7ke+PhAM/Ssg0dlxUUHCHh0dN9d5Psjh7cQXf9h3fJ/L9o08/g8cefwxXl68YgDJWSx1o2jh8GQscO9cEjjvbfIRQ7UNpZ+On0QSxIsScGtMMAlrGXiEUIUghWJaZM3iSU6a8fS6DifIEKqUK9i/M4NSNN+PW2+8UM1aOnlivu4wUwqaMDOhAEZMWS5Z2WaQI2wzyNZzRqw3j5BAurmWwGN6akFD70L5TG3EjjFBGpmhJn/Y5ZMREDSyOn7Sikys4D4Fs/uSP/9ukpKJwMk4oUgPk6FJ5WQztIyU0EhvipzG0cIaJr7iQLKnYtNVqK8eayeHVy1t45zf+n/jkpz+F8+cuaCe3O1TpVpyuHUYO1oi44EkT7TjPJXsFRnjd8uG1K6nGBhh4sZyx12yhtcjK8VqJsNlHI7jF38eFaFybjAtHwKb58gQI1jA+J4tmfmYex6+5BtccPmDeL3qkfouuJIFNzLHV7vTiwVjgKPYzgQzv2ahFgmY7lsAJuJNzTY89dr9COdaBZ4NGxXsa8ZGOXEC8xrBJI0XYlvyBX//Vn0zajQYmq+Sb9QxtoipKvG56wNJQBu4GBngkotooedJEZ+QtkqFhD6b0Jx2GXBk7/RKefv5ZrG1uIDUw4iCxbNpk2maFcz7rsYBhm2PhQtWG6chI4o0LpyyYCmK4iJT0XY41d7+WX3YuhVTGhGfcnsf3sdvHfYBIJ3Lxc1TtBZL3c0bu4KISfi2X5eFP5LK47fQNmJmwShBqiBFU6hUZdLgshbtrPhgDBz4fwEqMyWrJrALGVLz5TwRvbOGNI9DvGRaiOfDUcrBc+DMxc23WD/3mB5LN7XVMVSYsC6UkeQqH9h/Bvn17MDU1o52aLVWMJeElran00PK+nabiPe5WOhgE8pP+EINCFc+/chYvv/yyUpO0J60mHTDzsBV6yNu23Rn2OB6Uv1eO2RhyI0+aP4loPyq8J2Y8MJanY+KBfAnpc7LguJMW34f61jXdU9+140b0I0TJF/EDZIj/M+WbR67AxFBJDpbsvfyeDMrFKrKpIfbNVnDztddKEzDC6QtYoa9jzQqIVyszSIoVee6OM3Ac0nhjPooVRXhRorho1q4EKdvhUTYdqePYHBIW2vVg5Xz6H/4k6XaZ5aIt6WN1dVWkAuKvlCLaHbryzIpJUl18xIPOpOTFmlonamRgQJLL4eJmGy+9+KKcLg6e3mGzaYjPSK0ZlVrvsV1kYU+kN7ngI+ryWDWE/C7PiZvN4mJzZB5aOcGBJsfE3VKioSliYcMsjNvzEDZG/0aiMEdIi6SEQxHFUkVZQC4UVaS0U8YBGAqiV8jksmkUc1nMVSq45aaTgobTXpJLZyvoybLPo1IdY+2qqsRLltR1watCtEPdQeYGi9DLtoQ5hTJhgp4jXrcwL/UXf/RLSqdQCsx+GrbLeqSwlLcAACAASURBVGVKEFWFpQB366t5MzpYVD9cSEuRplApl5CvLqJXrOCVl7+K7Z1tT/dZxobCwCR/qGsuWDgY8RASHKFK9PAt8xYPZ7nrFLIeUlAABfprt7CyMoMBQ5mITp1HF5LOz47b43FPPDJc4dD1B8zpm2PFCSSOzs8TFqbJylcqUum5gvVqSWjC+kaUVIHgwHqqsFxI8zrsygGeLGXx7ne8HSxl5D1VvizqtFWrBpUrtJIxTswkBMxqxY6SeOcAmh/i0qy/8dmiPs1dFqR+4xd+ILHuOlbiQlBBXQdy5FSToGDeLKmzQqpUOG/0YpHbvc0EXaFBfhKl/dfiqYc/j3q7hW6LjpgJCz9HDjZBei6MFtE5zrHrAgkL7jYHH4BNCIF2WYQXopsx+LTnlKOUIZ7kxQgeesX1YyG/NpwLTRM73cIWCwNDy1CdcxMYPFxEkiNzp4wkYzufQsD38FqCdj3lmvI0roiVFM52C1tXL+H2G6/DO9/5Ts/W2diJZ/Mlb97JFRKUsZKrCKtIkmDVjsHYHoV4XxjLqRv3PIAcRQS/9cs/rG1n5D9ic27nvPoiiuRMzbgO99KfiANbrR0MhxnsP/12/N3f/SUyDnZQOxiNyJiTzDoZB4w/m80Sb83VdYRtob7DBsm++w4Zt62pUH9qCUVfg8O3/HHs4PAFIqQLJ2/cRxjH2GMMDKG0WxyNE1qo3LLVUTHTx8RPJl9Chg4se9Kwhj2VQb1hiR9OGGu4FF4hjXTSQ7NeR7u2iU5tE//ym78JJ48ftbptItxO+DAGi5mRICMGrs4oRxx4gkwwGFUl6iRDiMpkcxuVNJFdUzLlv37wP2ixVZfsZD05JE67FewmgMOACM5vgP02EH4uwczR2/DYc1/F6tIr9neVsUTLJ7NrDCcaDcKmJDdSEMx+M24OdR12VWqIVZNy4v7/VYzane5lWu2MIUtc7FDX4Wz972x0/C7s9bizpmuz84SXB+k6LlhRCWI8vDzSuRISpRfJiSvK8TThNAezXGE+voE+bWmvo2Cwtn4VrfqWHLef+g8/aowez9eP8geROxBl2KBYsW2UhevLUMlNUbxOyNXyF7wW7z1OqwoMI/WhX/mhJBZUgIX3BIv6qmBXWALe0pPuH5tXyf+dFvLH34L7P/a3SIYNDZxMC8F3TMnxMwJDDPK02m4Lk0wN79rmcFSsPHfXWePYYkxRQWnjME63TJbHcKGmww+I3bp7bbNv8dz83jJ4RpDQriSvzZEv+QxU105CMNvpoU62YOYuV0A6V0QhVxSIwQVniljz0++jTnIGG24NE2ytLmN7ZxXpwRA/+1M/6R0d6MgydUmVbpskiBARchl2bhiZxeduucliCQfWKckjs0aNOCTjN4/Ub/3iv08YQrCaIfhhu2GPYa8RAoUDZ5JvO55aodnroDZ5E557+CHUayvyUoOcR+FhJ0LtdudHEVMW0N8xcgFDMKk6955t4i15Eeo7FkEL57zvWLyAH9NZW0Q5bWMtu8a97XD2wqEZQZtj8Kny7EwFEqgcYdVWshTqn0V0NqHuw5C/njMiZrqQQy5rxREZr4ztscojGQgf315dRr2xjnwqg//4Yz/ila1dLSQXJgoNZJfFErW+K9FKLNp1EBs3pMyRNufnGZpsXj2/mgYGUh/8T9+nKk5WPoSBskm3zJDZM8szx1dzZAylYrhEqtLmxLV49itfRLOxpsExqWDCYzsyYL4g9wVRn5+ntgjnKHZbnoUEASOSOapWGUZb4kv23MEVLTpBBu4cx8/HwZH4Pr4K2Bgj/MeCh6NmKt18F4Ieso8Ou45/TuPwWD6XLig0Yx6/n5D4UGLnS5RLJEZah0JmyQrZNDZXCRevo5jJ4Sd++AcdLbPuipayNAdTIIwDMOGoKUHkfsS4mQptFlrMwBbWirtW5dxxsWUPnPX5tZ5qEP/dr3fyn4Hz2o3suNDpY/KGd+Lxzz+AixdeRNY9VO5wMk0M6SJD1CoUgjhnHja9cgM1DB40ocupoJBCZa42Q6qAT0cPOQb6K+4nNjDWqoPPFQscKjoctPHnDOctBM5UqAmVFbfbDhnVTHmZrqIRvx93eIoOWybHDJChXKRZFyc1hiafvdVGIZfG9toyavUNlHJ5/NSP/ahrNIIO1Epm7zkHyi94nbnh6bYfd5MlZsi4uagNhNx5HkB22pHMqC9P/ebPvz/hgKluwhGKna3p9fAodpOBdmzlZIxKJgJanT5Ofv2343P/9ABeefZRZNJUw6wVtvJdAhGhsg0T52TKuzDKMLsVhN11hEwqyEOvcDYi2c8HkkMXjXr4wKL5WLw5WgDPzH2tGh/f9eO7elfr2K6WgIAolJVARdGinM+BJzBYo6XSHysglLOWNgHJ5stC3bhjudDKQPXbqG2to1nbUi79R37g+1+jrYLepDVx51g5ctcsMUYrLdrtLxsmRqGqGEAUxF1QSprhN37ue9VAx+LBcFJMYsxT3m2foR3mHYXDzhK9ajVauO6d34Gnn3gWzz/xJXQ77NhgHuHkpBXDGxZuVRoR+1kmJ6V8dixQ5K3lhHmMKiKe57HNSfOiAW8UQGecjk/kt83W72a75FX/bwraQ+XLprmDE9/H5JFLxvdxh4emkJD3jDOnZxqShWPv0SKl89o8SOeQVTtN443xvflsVqyXTquOublZfO93faelI51PF4Idv4tx8e/jYwuTE8JhPpDVltNB5L2ClxDzl/qVD/w7lexavbEjVGNNVqN6kQ8RN+CFFhYWwBYQxWIeSSaHzuQJnLu8ise/8KAexpy6IeYXZ71wwOyWhVKmqqimVNM84lPvdn+IQgOOje0raYMCD4/sFheedj0ctkhphoqORY5F3Q0jvZPDGGWY4+JzRQgY6jBaXkdnhQA4ct5zRmgZm+8RIVSM7w1o046sSWPSnzVGSqrLxj/b4udff/11+OEf/EFfbGO2hJNq/lHAqJ5p9HZlaTmHDDONYxa1cdS6mltH56h9ogpUc/BLP/OdymczbolYkzsnVGXknMnbYq8RPvSo1ssTCCwZquX24NIO8MTnP4Mrly+OgILyBInwjEENFQpEzXZL3hrTpq2nWBD+xu1sOGJmUkIhW2Jf2ACT/DExY4iZdp+XvgYuEJM5vtPDHkc0EL5DaAIrKjRGy8jR89BHvVy8dZeySwlZKabOuU4K1cQxy6g0R/dXjqAuuPRd73o3/vk3vHdMjTMnb+2/FPJGaOpOqXnf5mkr7aww2Xh9Rllwe27fjHiC8WypX/zpf5swSJeKYTG351S5uATuc85bjpCF8bEe2u1jmlNNzzFVwvnuNB556LO48NWXkMomyInUDiwszo2AFAvx0t5vu6ydHdpDu9ix8NiNoY7DpBAXd1/JAIxUImGx1N5uY55Q5fE1JinEJa7Pn2PXCuN3vH40qeS5ec45FtxqoS29Glg2+WEquqcL7tGCqWAjTrCXaTTwEVU6ncKHPvQhlUiHmRPbhw7pWBp2V0CtBp73NQ3rFC0nMHCiJdzeL2a0+B45aSwf+In/OyFXiv27SbpXB6IRMS9tOLSyLN7wLpIQUYutBu9ZdIcJznXm8ORXHsa5l55Ft99GOrHWUlNTE1LZFDcurrzMPqE9a0jL3msGtJiHHwAHB8hdoqY3rE5UV0Dz3G3X7qpxg3stsRI7OhY6zAavN55wGXfUYnF31WhMqoFIRtm1/IBSvS41I+dJZLY0uh0nGoYdbvdUkkP1ru5L0XigVMQHP/hBoYCGVnr1ihMTuKjGOHGKkYeD+tmTM0ZiMAatSIteVGkIk7FUhcwpu5hC6o9/9/9J1HzVS2eEgdDekBJM58JPGMhmmOVJI3EUiQsshIv9vAg2II2vrnbxwvPP4qlHviSCvvBqVmeW2LzVPPKYVLOPhhoV8+wRYrxyld96OBOLEwLAWnH+jTtZsbtHBru7w9E9j+3Gw6zxRRy/7tdqgLh3CA0xcj4rd4xahgRI4YsgJ4222Om84deElookje1QFjQaF+/EyWvwH37sx91OBxXZulOpfwrDWmbt1FLL1HIIp1KqhRyGHWeiOOql4zjU9M+aBFohgiGRCls/9td/mBTLRWTUSwQCBZKEKTfr2zGi73oFQ3qw60QpNEmxwRtj3DSu1od48atn8ehDD2B1ZWmUiy6W8ihPGJPFvHEvuAtb64sbPkOYknEHSw/oD0xvM4SGYyTGzOvGZHxtDB3OllKKXgfN7yMBIgFyGz+uBew6VuhOSFRC5zy34I0x2aNIIW190MI+mgOaRTIIO2u5ezstIY1f//VfwczU9AhsspbfFs4JKQvbzHvGbg/AhbaakYznrpW/GrP1u2RM3ziujVMPff5+IX9q0KL2y757vGwm3H2Lei0nPY4hy6HxdFo/yeHxVy7jSw/8Iy6++qKpmEwa+VxWhQfRp4XccF5OdUjFDLpt6xca6pkTHs1aaU85iVTz47tw3KabJTPHJUKRWPiv1RKx2/lc4/cct7OKSZ0gEOxPYeXBb1NDH2eQuhYZjzLsnhmFWeY505QbCklG7Xd/93fjDW94nXPw9FcRMGge4h7RrYmXFzVpnA3rfPQe07DUKS64chIpcKo5G8rsGcnRk1kPP/JgQk/R0pykYxqYMALhnWLbb1uXWz6keeNx8k5KD8JS3VyuhOcuruIrX3wQLz39+AgUoNQyfjS8mXnznpAhkeDTAyR9CxnGqzPi4aJOy0AZE7RQw5EsYYO+r0XG4vOhHcIPCDX7tSp+3L6H4IzfS8wVz+Pzmv2ehakhMCEs0cFR3HkdTZHHgYMH8KZ77sGdd95h+RWRRUwTRe6BZkkOn0cQ0UslFt9Ewtil9PLDWbOMJVG0XWbqeMtt81E8qfT5z9+fsBMv7aHVPRmfigNSAl0XIqmcRXQseLOeXqxgZH5a2DbhTZ2pUcCVtW18+nOfw/NPPKLUpXUpsm75LMfhBLJVRKdjvcJZE8XidoUT8jDNQYtJCE95F3TZ7T8mQqEcOscH8plRV4TAv3fBEXOc+IpESahsmYgxtC3MQGiPuHcsfpiC2P1a9HYfe/fuxfu///2iHhsM5Pdy+rAEMG3PZxTh3TGxr7uIEuwU6Y3reV+WRRlgYk2AeS91qnAiYtC2rJWJbRoCQcIlIivorcVSD372kwmzVjqRJ2vdh1l7FQDEoGt4axSuST2pgsT7blLd+SEtjDFT6QKefOUM7v/E36Fe2xoxIwnAWO/SrOq2u11SZ62WizaXLzEyHXCJiYoJjh0+PtFy1EZJGh65YDZzHIXiIkZIFRBo7HK+N8xULGjYXA1ojIgYAjCeJ45dd8cdd+DffNu3e67AKjZpQ6PG21SpF+2JXGmYugmZVW8QhwgnkjtcvD0nDHLhtHO9k4L5GAyTdxeVi22JKzp0Rhahn0EBoGoX+vfpf/ibJM3QqdPWLstn85icncYLzz6FYcIwjJBnFXv37ZHtaNU3MUgySGVYrZlHZgDkK2wIYwxPqphXlrfw9x/9G6wuLwlDZ5E4ww+q6Xqt7g3r2BfNeoMOKInOlFEI70kRIy8ECXG3VktxtZzH6LliNnZ0ksAYOTGw5JjIWAC+N6jIdoSUYf29riF8/G9CbdpGCQ5f/NAEHCfr2n7mJ39KY2ZhgHqjD/qqTbfEhqVbWYynpvYD48rzFa1GuLBEIlUbzoZ9Y3kBnVDk7SrDbBCNMzqxaYg0mUHhs+ikBeMPcvz0j4zFk0Lqr/78D5Lq9Ax63bYkgdX611x7Eg/d/wkcP3EKi/sO4+WXX0Q+m8aBw0fx8tOP4/ipm3DxygomJyZw6dXnkJ+YQc/JJCwiT+XzuLzVwSMPfUYdE4kzVCtV84QdoCB0yvBASJDiCqtdGn+Zat/9XahNBXoKKSJDZHlmkiNjUUMtj9vmXe+eMazVnekeHpoY08N7sPjC8prjsWqo0sgw/b8/87OYqU6pw7HUvldi8Hk4FoavfFajEVGT2PtCg9gzMS9hVCRRmdzzj0NtKDChUaTxmPpVBMDuzz2rvuUpB+xVquY6lofv+r34GYFVH/nw/0hm5mbVe2t6egoXzp3DnXe/Dl/8p0+qo++RU7dgmcXvVy/h+tN34IXnnsDJ625Coz3EwsIcHn3gozhx+s0oqEVFHfv278fTX7of5cM34S8+/GEsXVpCPp9RO6geC/ac6cLJ4aFkQnpiQcc93rGFJl4VvTsNVCHQE0wWS4wYkGKCQVNjDppXcnqXYOamJQyBKbN6xc/90G7lzus6Bz1Sq9EiOrEMHR1F64OSYHJqGj/3sz+npEh446ERgnI1KgOWX8IerB3tYIJNpkms0Q0PYlPNupMuIoyjsLIxACneuXzBKkM8VCQMbfQuo25Rm/R40kGpKN+l06xbXThbpdCGs/PC3MI8dra3MT+/gLOvfhU3n74Vzz/5KNqNbVx7+xsx7PZx5sUnceTkDUpyFEtVzC4eQnlyAk9+7mOYmN2L/Ueu02IfO3YUjz7wcUzuO4LOsICP/t1HUaMq8dZV9DKFJMkeGUU2asis04QdTmbVIl5HNebIjHunEarJ3ku1pcSQMTVoFY2aPDXX3c1ta4d7VYWS+4RMM1YjxYlnSMjvdz16i5F5P3rXFk7mVaX5rne+Gwf37hsldsLBJFeNY1LbixZPTjCba9i4naQQfk803+NX7sDwJaiGubhsTBC+C7/yOjqZIA1t0si9B6N0e3vHyCNk/uq4Spbx9pD664/8fjIzO6u2FWxNwSTG8ZPX4crFC1i7/CoOXH8bFucW8NzjX0B5eg6TlUnUG01cc/I00rkMnvvypzTA46ffpAXau/8AXnziATRrNRw59UbMLsxic2MLTz76EL789BksXb6sXWGevrMynMkSB4lG191oWZl4q0h+jhQqPgiPfeAujxYUVu/sPcZGoIsd8Cq1SJUfdc1OiJQqde+fAIXh60Md+CoMWiR9o/bypTiYcbP4vEAubQ1riO2Hz3H06FHccMONygqye1TUG/EZFNuzOW+vp13ISwVMSgRRi+LnpfCrteMsqgcMhZj1d1w0CZu34OTOpkIzSDnB7MysasXYnSoO4su62Uj99V/+j4TF6LWdOqqTVaxeXcbhoyewvbmGK2efw+yBa3H0+LV48ckvoj8E9u87iq3aNvYdOI7iRBlfffJzaOxs4/ANd6HEHT87iwuvPouNy69i7vAp7D98rR7wxScfwKByAB/72Mdw+fKyqb2BdTgO+0Xpj7CEoQapwnzIyLZx8Ny1Ukm0/Q5YyJN2gbFsmLXVjOI4LZYxHV6T16ZajyTQbjLFD5rLG7NVbBSP7y0c9DCR2kQcNW8G7zn3cNCII3CcLHZg/7SJsp1lwrCM5nHYbSmKoa9jdKs0+sMu7Y4EgYe55Qs2N9T/1g/V6r7Y+ULOGokjjZqKKNVpiTVfbPbXrKPJDlM6Xbfgba0HSP35n/5uwqpEa59cBM+Xmp1flId86ZXnUJpawPEbbsH5l55Rw/mFPYfEpZqc2YuFxUWce/ExbK1cxsTiMezZd1iLvXzxPNYvP4t0YQLX3vI2dSB89bkvoNnq4vMvLeP5xx8fqR9BmNHPVOwV271c5JKfFMDfaZFzu0kaIWV+Qq86D3i2R4APTxQKh8lLYwngMOHCtKrRjiyhEWaBqcoAddQtSr3COXF2hgfbVZl9NB+DZT8sMOQiqZuTzibxhgEOdFBQeF/ZVPfCC/kSDh44iONH9mNl+SoOHTupnnArK1dRmShhdfmiHK3DR67BytUVnXaYKxZVhdlt1sVJLzAbmStg2GubZnNIt1CqamytTgvVShkNP6lPWolz9Vd/9jtJvkxyoDVutzjVmrGtXDwnZujJG2/F8tIFbK0sY2ZxrwSjOr2gU/GuXjqLnaUzQLGKhYPXYnZ2Adubq1h69REMBykcOf1mdUQ899LjaO9sYjs7j4985K9Q11FN5pUyZOFXWtp9+/Yr3hYzxI8nZlTGn6lo1ZMz2l97VaaFFlSnFk7xWlJvcaY2QaOx46oihqeaFN3XF5+2UPdxhzHUvFKq7jCypo0aYZzUEeDLOFizGzNb7xQV5jmGoNjeyZgEnt56772YmpyS8DY2LmNicg7XnLwJly+fxc76KvYcPIyt1VVkEx4ydxUz+49jbn4R68vn0ajtoFouQIfjFLhBymh3Gug0a+i1TdAIdnE+Un/xJ/8lId+Z+LUC+X5f9pDhQH19BcNUGvsOn1B/tPUrl5EpltUMNpUpYe/ePdhYX8ba2efFtZo7eB0W9hzAsN/Buee/qCMo9p28HYcOn8CVSy9j+/IZJOVF/PnH78eFM+fQ7Rnezfvu3bcfh09ci/m5eeRy1sEvuv30O9bnrMQDYZx2LBXrP3Px5HQZqXrk8Qu8oPCy+I5xrjea5zPy89FFOECX8URKNKoNgYmkCSnBStHGkY9RPDiWw+Z4IlY3xGs3JByhdrLhPF/T4F8ybCmQxw7OYX7vIdz9unuwvrKEKxfPYe+hw6htbKDb3NKc7T16E0rVKVw5/zLQazGzquKLfGUGM/OL2NlclZlg10rejzSpEos1//T3fzkR31nF3XYqnzrRF/LoNJuC6fbsPyJbsaZMFoeWRbZYxsL8HkFzK+eeV0gxufcYFvcfE3l96dXHsbO5ganFAzh6/BbU6ptYeuUZtb185lIT93/606jvbKDR6eOHfuKnUW8P0B9aX/B+t62meYwfCXiwebwWiIiR0CnGqhazdhjX09apM7E1j+VxVRFeqcpFaUMrciAwRE1g6VaDaMPTDR5XcMnioNnIkAmNU7WqMWIDsKHNpcPJ8NLOFfXTdrx8KFp18/ddnnnqfcfl7XtmXGeSqZdMTxSmQwcP4Z7X3Yna5oaAm15vRwvOse+95laZ3NrmEmqbV9H1as7yzF6kszwQponWzgpSgz62eYpvZRKTc3uQ+uPf+/kknS2gQM/RWQ18eC5Kp832WAkmpxcUpNNpo//KTZUrTmDf3gMCA66cfQHDfhPpyjwOHL4OxXwJaxdfwtrVcyhOT+PaU2/ULl8+/6zUYbtyBL/727+NlbU1fNcP/LjKaLa260ilzYwQwKF3WSa/LUlEqqCw8RpimGZJY2L/MaYQ+xh2efRCH722N9cbU8uWGrXr2kIbYNwmsqdG+EaJChiWX62Az1pYRIYvgI02QxgnSQaiJWqSw7KMcdXbTYV90aXJEiZ23rbF/vZ9HMhqHRSkPVRTwTH1UC0V8N6vvw95HajXQnNnW4zUvcdulTlbXzmP+tZVdFtNadvS9B6Z1+3NDaBXw9ryZWvik6RQnV1E6g9/62cSNpnLuo1MeUaF8KBaMOoQlylkeUh3r42GmCZZtdCYmJyRyqfdbuysI5cvYe/hU4JXV69exOblV8XeYAjGU9uvnHse9Z1VzB64Dn/2N5/EiVM3Y3pxn45n1IEvLEFVKGPg/wghEzrURSGbt3M1szxkhXGmgShpgjE89LxnXYLZs7TXZN6YkGRXNdGKad37p9dPDRKN9tSvLE+wYjCCcFlxysW26CCl7gahBfg7zoslM6xsmDvbnD5r6MfFEA7gvcKjC4Oa0PF0AF7DY2p+r2ILfc5r5HrWFLA6kcc3vOPt6LcaGPa7SJcncOyaWzBIp7B+5Ry2rlxgcY5M4fzB61EqTmCYdFDbWMba1SWFqRSwyvQCUn/wwf+YkKhAiaItYvsIhhNsXqf2Dil6x1UZeXYopoqU9BdLKFen5KVurS+hV6/JBMzuP475hUX1DVu/8JIWYM+J27G4cABXzjyPVnML5YlpPLvcRXlmDp2etd8S89QXkhk224l+aqA7TMzMyXazl6p77oasWSUoEyqceDaHS3kbCi4YPVnZzYT/DeumqdFB65HedWKAWlzJy/YjLbwgYChTMlCOOrSAOYK77BtpAbD7RFvevPkJ1pGY17TkhrUXCdqQBMd9iPBfDDJmVScPaAW+5Rvfi/SgZ+ZtagYHDl6PHoZYv3IejbUr6LGWPJNBdeGYmgT3ei1sXL2IAR01xuoTFZSn5pD6g1/70YROGNtIkFrERVZK06sp1JvDKx0M+7W0W5LKYnJ6CplcEd1WDTsbqzqFoDp/AAcOHlEP1NXzz7PfFqb2X4vZvfuxvXYVm8vn1PZyYt9NuLTdwOb6ttAuJUl27LhFmgp77Ta5s7DL6sO5s4lghSMU5bWMyyWILhQcL71QCpESFd6ey0piTCtQGFhTpSMn/WgK4eXMoHmKUhAoETcJgZU80RsPx5Dawzh1LHw0UkR49LxnOHcBgYawBFrGnyk00gxjPVzlHWWzeM+9b0C1lLPqmvwk9h44KlOyevkVNLau2rNkM6jOHQZDO4ZrO5uX0anXrCd8Lo+JyWmk/tsvfH/CKgZCRTlWIFKUrNLLzqygM5GyKkURERkzisGWQ5GdFgoTGPSaaNW20Go0QCeBi02MdvX8CwoBJhaO4NCx42g2a1i9+AobV6By4HpcqvWwvr5lZaaqELWJ4iIrJednafG+ERLxIQmSiEbknCum9Pi5qNfm7jOWqhMTiaDpyGg7tkH88yGUk9fnlIywMLA7sG4S2ZQVshMjUNJDXYzICvW0qHvhhoFbXpq7qOskD2kYp2AFeV+dFb6mTCcSKiGMwaAJX4Ff3/2W12P/4qzWZXrxKKbmFiVcq5dfRae2au23CnlMzh9BuWTtvzdWz4JUETmZ6Swq0zNIfeg/fXcigqHjyAmbzbK7AltLyzYzCc4qA3c2VFCQIJPn+ZhF2XpOXmN7045xqlaxsO+ornHlwsvoNtaQKc7iwPEbJCjrV86i3+mjtHgMm/2iuFRXr1wxRMhPD7BeXl0hZOEpR1ZMRx555YUQLSpELz5Uk9eoBGU9eJ4q11RmxOKWnuTCkCnCyfDzNpyDprM0WJbkvdA73ThegpSfFnLUbqQww05D4PUUQXS6fta3lSSHLQ8nLnZ34O2RJo0jKFyVuYDasVFxxOV77nsD9sxO6muDMwAAIABJREFUSkUX5w5g3+IBLeLm1bOobSxZGXRviPk9R1GZmsH21ibQ21I0pANwGx39PvVbP/sd1AFyoDgwNokXu8MdDJaeplM5JDnLVVN9m9NCmnAJ7A+mZCNVx9YWUrk8Fg8eEzy4fPEVNLeuIElP4NgN7kEunUW31UV25iBa2WnVSa0sL2uRGA9zt6lGKTPEsD806JBN5ssT4IlEskHecC8otOwWQc+a0Kd2ijxj8uDN+7bOidYWK5L+dK7YYpMTpaSHs2aiSWyUNxGv5vENwx6dKPY86arUNpoXtPtdMw/eKIj4dajigIEjPx8xdhAX6DyFoxhCbQ1sR2WaEuy3vek2LXapNIGpfddgbnpBuYzNlbMYtLcUmRQmJjE1sx/FiSo67SZWll5B3rVVNlfEgIWHH/rAdyZiOaQtO5RmGwmiUZ6xIQKsGmVWJqZTVmzOXaiOPEWUJspuuwaob22LZTo9u4Dq3CK21y6jvrksFHnx0CmUKhWsXTmPZn0HufIc2qX9SkRs7WwpyU71yyOQAokKtRyn+ubyhosTdaKNJVOTqUL5QGOlM2Ez6UOojIZwqx+uqkn1BjTMGFEzWJ8XClZeuLLial88xqqETOkEqTmfU5iUVnXnyrxpO4SdziCzXJEAEVbujFad3R1HZYjM4Od8e8M6TmQc16gx+CE0//xdb0KF53snKew7dBIL83sl1Mvnn0ONNps59HQWE7P7VRde21lDNunIBxLUW5kStzD1X372OxOzOVb0zZBLaFTBHDX2CleaMLFQQkcTqNk5Y/Gy7IF1sx+q9zYHWChXMLfvIHrNbaxcflU2ZfHIDZiZWcT2+pL6irAJfXfqGvkKXGweDcFqTsbtUaHoLbSlVjmZhFE5JmLcUc9katGQNf7nwgX9iMQJ29nBJPXKEYV5u6fvMU896HfkeCrP7nGwbDeb1PJ0wFJeKBfrzsLDVt83liA7kKJkhjtYTGTQOYquhMYPYzLeqFfRwcJy7pGPtwaC8iGcEcr+qd/yjW9DliatWMb8PvO4eZrP1sqrqG+tWPuNdA5z+46qgrTZ2EK7tqbjP3QC4YB14hWkfutnvt11hpXQBhtEh6MzvFExALnZWaTzVn8sJiSTD7Tn5K3xZKC8nYqrcy1KE5if36sdtXb5FbFVJvccxszcgjr4s3mMSIvlEwpVOmxDUa/LuYlcbuDVlvWx8ETd/dkf1Q84CcZKwkXgJDsi1uq27TQgr57kLlVhuoTaGTHe2sPOv+buMz67cs6eCrW4Oiv8nCRJOX19rzrReR5RgUJBs8pSMkeiEQl3KtOl7CYch89F01i69jI3znc3X4MttqzDAgWHWmeyMoH3vO1OTFan0RoMcejoKVQmJrFT28L60lfR7zYFnKTSZWlT9UEb9pB0G1hauiRNUixPYDhII/WbP/2vTY37ohqldRdW1NmWKo/M0OCpFFUYsnho1geMks42URaCMITIozI5h8rkJJbOP492s4nKwkHMzC5qR+6sLVviYvpa9NgxMWV8rJ4X64fHysmXSiY1iBAn04I6e9MSGNwd3Fl0jnhdlsFGaSwFNc77oAqLuF2qUud/GeOFcTX/RuFmbRuJAqq58lBqBIl6fM2TiMPmmrnY7aYcp/Ba41w3LXQO++yVZJTrqLSMggdreGMLLSrx6IjqtDTD1FQV/8c736S5nZxbxNTsfoVXPDu7sXEJnXZNglyd2oPK7KLYNIxqCKrwpGSmr3fqdZRLk9zZ36Fi/MjcREDPiVD44+CCtX5iC1s/c1pnhDA+ZjuJtJrCMUHP9BxDNoIwk/ML2GKXgc01ZAtF7D10UiqPP7MNZmX/ddjqG57MhHuj6Uc9DW0RR6GKdiorTzpIuEu7hpUTEVP7KLbS9J7oXLxI6PBZomCdpkjtuHg3jdvqrWk+goIbTQLkoHq7jvGwyey9dX7UGVrcJN4dOUgQ/MoIYLz/anjaUZAoCpXrU+5sgwGN2B9IG1uAc17vufs0juxbtM2RLePwsetFaNje2cTm1XPotWqoN9uYXdiPdHZCm6DXb2NjdUmhqDUw4Jrlkfq1n/y/VJ8ttTFWlmq4MGucrMsfU53y1kX5zWHo3QJ1oEqprF1ON39re0tYNosGipOzysisLZ1DtlDC/P6junnS62Fnex2Ti4exmSygM+Ahbzy1hhMPdFpNLabSrCsrQsbUUbHfwvbahtSikKiehU089ti47XZS4Hi1pdGS/MSByIJleaotbbkVHhi4stulwPhscYCLV0+6lpFH7WQ/2d047H3sFEE7etF4YSE0VmCw26dVrFvaZTpq6pC4W8BHLcCzWk7fcho3nziMTqsmBK5QncUij+FImGhpY3PlPHrNGjvJoDqziInKnO7RaO6g19rRQQHUVKRIsX9b6hd+9F8RNbbzPoTC++GnnguWeo/KSTVbpUfMHizehsIPbGOF8GR1Uk1pq1PTlldOpTAzN4+rF8+jN+xg76HrpHImiadfWcLk7CLWM3tF9WFMScePue0aKTU6M2tTCRFmgsjk5RENje0dqXvBlElw2g1vHq9uDApSLLx2ZZza5+UycVipOh6JyMIODFGf6ScI+yLuxskegqrbgrFbuctD3ZN9kuJCC//uW6/vsb7qTGqIaDFioBikGqzVfDaDt977Nhw5ehS5BNjavKjsI9X9/IETmJyeQ2o4lBrfuHpOY6YWzZd4tGNFgkuKdrOxiWG3Y4fJcjMih9Sbbj2U3H76JuxZnEW5wGMgbGcYsmTHOUnL+JlVVNuSfB4xIftt8CV42MpE2equqxXtNDam3X/oEFaXltDpt7D/AFG0JiqTU9hcX0OhmMdw6jp0kBOjIzhZdNSIVtG2Moxpt5totWroNNtqkcm/G1drt8JDp+xSCBMoHAv4MXaptFLWIFYdqRB9x7UQdppwf2AkiqhBD7ttTiNtOyfDW2RFoTyv56Wz0jKEPcWMTsk5ox7ghomW21UeLyV2ib2OHz2Kd73rnTrakX7H8089La0wOTcrz7+2eRk7W5tqaLD/6CkU6FUnJG3WsL58Fjwsjru2VJkBUkZy5GIPBy0Mve1GVwfDVZC65YYDyc52DZ1uH3vnp7BvYdKci2Qg7teeuTmxKKpVghpMORpRwFgtwqasFbPjuJwoeucKHZIheEYlJW91dQULe/ag3e6iPDktQiL9vurCYaxiHgl3sLJUHaUtZZO7jFlbaDUbqO1s6G+M5UmOCOyZE0Shi1NpFaOn2bynjEabJTNZxc/WoZ+JClOlPG6AgsoiCNavjRIgsJpoU+27rUWCjCDVOxiiFGd48z00H96TLCNUz2JrhWR+AnAqm0elmMVEtYiDC3tx/fU36Pip8ClUxpMCnnj0EQlloVpFv9XC1tplgGeDF4ooLxwWKbRR20aztYN2bUtzRH8qW6yiVK7aCcHtJrrtJhKCQATApE2ySH3vv7o3YTqvR8eDXYa9+ZyqCr0/mb7qRAErLdGBLf2hFnl6ahJ79u7RQSqGaLGSgtUQrGe2Qv04TqJa5Yl5fRQqVSFOxL6LE5PoVo+h1UuBNWeKibsdLQ4dL8boGxtrGrg87xbP/zLcOcJEqWOPkYm4EeUSEZD1awXrrM+QjQfAqgyHKFjBCIUsT2ZhgEgDNGEeOAU3OxbZ4E1r0MvPTfL0PyJnLhhWnsPr28HqFMZKtYo98wuyvRN54hCb6LR64gIUJmZxww03jLo+EKmjKfvyF76AieokSpOTWuy15fNqbstoZ/bQtfrabtaxvrGiEJbRMdkz1akF7XpD69qq8GFYxnFIjdP3+vkf+iZtEjZmV6rNCXW0wZwk4b7qprRbtald5z1MlaPyqg4V+fnpPTOzM7j2uuvEqCAIYIOwDj4E7SNVqQashTkkU0f1WcbqFBR+JQOD8XOzuY1+u6OfyaYUB9pP9RXgIgDD2leJBOAn7vCe6YxVTPa7BF94CkBJlaOBgKnvJ59HqVbadfNfmC3Ty7NbnFUlJzy2Vh8G92tYp8Wdye4Kx48dU/NZ1p2RYXLoyDVoNxs498LjSPptEGsvTC6iNDGtkwXjUHoWPfL5udiV6pTCrPWVZdRWz9uclWew9+Bx45HvbIrlQ4iaY2r3eiiXp1Am7yCblT3vd5mOrqtdds6Zralf+YlvVehFhUz4Ubli5oVVAdGjhTJnw20UmV4CKFxN8fd2Gp1liSIG5c6k/TLbbwT9bsfO/5pfXJQ22L9/vzx3kh6Ge06LVkumZiQSqKLIrWq0ttDheZs847vZsF2tQ8GNzMAXcXsKJl+BSRND77Pdh0jypFsVBcwwNOFY5ZiNjk00Z288V82Ja+zU7JgI1rn5ATlk41II+PXUtdfhmmuuwebWGmZn5zAxUcX66jIaNfLF+rjx1rtECrx85ln0W3XNyfz+48gVyzh06JA0DL3xKGp89OGH1fF4Ye9BXL54Dq3NS1aDXZzGgaMnNY9rq8syZdnUAM1GU2dwZrLkBvoZpMOekk6N+rZiciat5KP815//ziSqIuwQUivoppo2NTeCeXczSqPOu+pY7b834ELagQkJP/vLSkkNmaOU8e+0pXSoKCjqMcJMenU/7nnft6Pf2UGjZWgWsd3hsCe8emdjw8kTLQmWtWvmrjWP02yxOZb8T4I+zzmhGTFP2QiJKrLzDglBPxpRguh3iOPmJ+QxqZKy9GppghqqjLfde69ds83zQbMoVytaTFasVqozow5Q3HV0Lq+/5Q70Wh1x6evbV6U5D5+4VZNPPjmdVDsdyMptv/DQQ5jU4Xd7sbWxgtrVc6i1apicP6bUMcda49mpTXaeaongQLw+V54VtVspzWSI7Y2r5tekmYqeMELGf/9F9kET3OMkPe/d4VxsoWVaLMNwhdCovYNpOU2hkhCEuaPO2tpRmJPDybfLqwGxeox6aa4awQzVpyWXTuPU130LtjpsoleX3SNEyd5xW5tb2FhdQTLoOH5uxEIuaqdDLNwiAnnebPQeDVr7xLG9/4rCoYHIlJEGDWhW2pr0q4nyqE6d5ufmm2/GwX3k0PdF0ZXjxRMH+fBeU85Qi1jC6soVHSBPUn5UuzS3N3HkhtO4dPY8Bt06NtcuCTy68dZ7sF3bxpEjR3RSImFTWhCO60uf/zymZuYwNbuIrY1VbC29it6wh5m9J7Bn7wHVfK1dPS+NOzs3g1aTMHMH+cqsauTps2ysr6K5sy56mBrv8Yhp+kh/8ts/4H3QbCFUye8Hh9mC+lGAYyfDKhRLeeMcnbgzVP438F1CjwJivGVlnE1l8pSo97ZMgxPuGPqo9CYzgeqJN2qhGVq0CBgM+qpDI6mOtCjmzDfW1zA7M6NDaKKihF2XVP/k7TEMJCGyV1S8ywklXYgPTRvLF0/lLZQKKGSyuPGGG/Du9/4LhXWdTl0EfkPlGBV0lQ3kiwwcqnU+Kz1fmbp0GitLlzC7Z49OGZC6L2Rx9cJFXHPtdVheXkKqR422g6Tfwb6jp2RCWFBRLtuYTY0n+MKDn8P0zCIq07No19ewdO6ryoQdPH6bPPJOc0sHwHaHwPTstNLK/V4TufIMZmfmNa619avi3ak8macPq8Chi9SHf+dHRottIZf3J1HHwziT2k5mGLEhBe0ZnCreGp0kPyhUjEo/RMXAA5oDU+8Ww6Z1noaYrN7OcgSqDFNo5efQyS+g2W6g120pxqYd7zQaaDV3pKZ6ZL2y1kq4vbVfZm7aTtyzXR4ghQANP6ScEOTMzDTWV1clnG99y73Yu3efaYheG7fd9WbVk3OxL1+8LEHrdpog/6xcrSppEW1G5Cc455sTWd/awMziohaRqrY6VcXls2ex//BhrKxela/BoorlC6+iunAIczPzYHRSqfD4KFPj1C5c7AOHjomHT01QX19Gq0Ou+M2YmZ7FkjgCqyhVyRGfx/bGhnh9E9N7MDU5q8UmgsYTkzkHC3v3iU7FRj+pD3/oRxPtwniZiR21QTYQwc/zEp4ah5fa7uBLB6V6laPgVe+sFDndKGS3YwYtAxSokmBFaQ1ChoYuDZmTTU1iY7OJrfqmKE47m+tsrYB2py6An+8jt9zgyzTyaibIrhAFUW/Z8oKeN5242s46zp05o5OD5YB5XzPrMgS0egNcunwF/+67vwf33PMmdfl/5pmnMTc9qaggSn051kbdNAjPqpYvkIJUJ/GAyWpVOALHUSpTnW5gbnYaV5eXsdNo4Prrr7fvazu4/ba7jSY9wR7ljAKsCPHBBx/EqVM3YG1tXdy+2uaqophD192qg1fPnXkG2QSY2seESB61zW3UN1cxtecgZqbnVQ1y9fIl60RZLBnbKE50+JPf/qEkCgREY/VWjdEPk7syXsJ5/Sxt6/tlQqKe2+y0pNaNFAw/US96aXpvci66drtfUI4Z0SQ/F5rHJUl4vM3ygWtuxeKho3j2madw4eISVq5exZXlS3Lc1Bd1dhYnr70OxWwa1UpJMXJc3zh4ea8qoZcgN13OA3ciNYQa1w/TaPUH+PgnPoFbbrkD//7934/6zjr+/u8/gce+8iVzbPw4BjmTxKjzBfHv6E2fOHlCLBoVEKiYzzooMKTiTQnt8kU0jZWdWyR4qClRWTa7Up2wolB30D73uc/h5MnrsHR5SVU4w14T/e4A+07cjG69jo218/IbZvYfFBeP8DFbWk/M7cXePQews7OB2tam5fRlwzkHnpn72z/8aanxAOwjTKKaVk9MERVYrWidjvRSQsEWNGykcrFjjdnMsTPnbVxpWBtn7zzgxxf1ujxxqCTkSCfg+HX3n7wVB/YfRKu2jVy5irnFPejq8BlDuRhFMDR76cmnlOyQifAyXFtb4/AG6udDdxKenxDkDNLBMAfCive9412oba7ghWeexSuvvjRKDgk1pBZKLEMXzeLJsKEfEXRg3mNyakr2mKElNYyYs/W6wkzGv9RGrVYPr3vDG9SEiLmJhKnWYYJHHn3UBHYwRLtZUyODZquDI8euxfLlC+g2a3JoF/fvw8b6ppVZnz+Lyfm9mJmdx9raFW2GcnXaDnuX752oKDD18T/9Oc96xaLEQRu2IHTVY+G4+GKMyMZ46exoMQ0UiMW1isZd+dC1YrZdnYcNZ77ZeG86ZXOUATp43e2YmZlDu76NVg+45uRJk3T2YvF66VaziacfeUSTZbVc5L7HgY8mbAGt8jMqDBiZJdvsSln2SKIs4u4336MzPK5cvIiVlSVD8lhPXSAtyzo5jkwQixG8S6OlVXkd4tI0N9ZhgYJAweDPtPkkVcq5K07ge97/flxz5JhCKAI/HOcjX3kEO7UaSjyLs93E1GRF9fB0tLrNBiaKOVXDTs/PY3V1HYcPH8aV82dQnl4Qf2Dl6iWU8gVx0phfiDPAei0u9of/s+9sSyJwN5jjZd0LvARaDlks+rhaJy4rmk5sei/U293NVNbet2t0wIqfejvWEE622lmgUTZz9NQd4kqz9HRzcxu33nan6EN9LwgkiEsy4PNPPAHjjscZnS6oLm3xe9M+u2duywt2fjzbhPLnm+5+HTavXMH66gq2ttcFCAlhcx5ZtJuyyfImc+54RuPa2OWMAthjbhxyVeTC1hq9Pk6dvg33ft3XabcGBflXf/VXsb25hTvvuh0zs9PSIoRl2W2KHZwD++dYGT9rnaghU8DUzDQ2NjbF0WPju+iwVC6woH8LqU/+5S9rZ4fKDRUbReheyTc6fZ04ehh9U6XehMa98dHnojmNfm9N9ETrkZ0mxkwN63XVbvt1cLiK3kzLnLjpbhRLRXD38nD1O+96I5JhV8QH+ges/OA1n+VikxDo6dlx8zFuRsxRsVMLOOlW62VsWXK3KLQ33nU31i9dxubGGhrNbSUQQiEpDeu9xSJEDWaqJYeM/x5HJGqR3dkN4CoqRukLTc0v4r63fb2gz26jJkH8h099SpwAopTtVlPPvr29uUtXJmihA+ZSgqzvu+8+1Ld3UCiXlG2k+aht76hogI6q2Dre/Sn16b/6oGlXV8dsnRFVhoq7YWCFuFGOhu2abtsZHCQJDeEcGcgSoIqlEE2VxiEzpt9JXrTT4Omhs5uQdxvy9OO1N98tpIxNbzc2d3DrbXcDSR+dtpEWCMgQwHjpxedEpzWYNHaupSo5vjixwMa/Cxrp++iE3DcTdPr1r8fy+fOqH6cTx6DTHDM7mUDM20gWceGdzCAz5R0gomOSiIuuScRC8ffaGEijmcBb3v4eVXU0t9Z03ccefxy1Rt2Yq85eVX23OkuRjGnnoZHvTu4AfQGdlUrT0TUYuNu2UwtOnDgpp3Bxcd5qyD71l7+h0Mt2HA8xsSZpRKFMPXtxwKhPib1P6tDroQlUkJkSXXCDdWEPz2YzfmqdN3qLUMwOHkvbGWx8qQGvgTH8/ckb7/TzNbjYNdxy613I8HRf2h9fbGLNr778guwcXxEh0GdQBYvzxU2VjqnwMSxAdeCevrrlDW/A0pkzKmC0fqm77bkoKrTB6tbsr3EUTjZ9LFctyFjQoh3hZEJj41AkkCvjbe94L7r1DWytXpEwPPfC83aWp1pVG8AVTXEZbYRGMg1h1SnBqOUCc/HJ3AmyhX5uNc0p/cSf/1qiRQ1P2rsKEQZUJkdlMFbgZ573bvM3O/PKbqgDUehgSQ17LjgcNnfOwlFidkgagR2FoxhdYZA5TKQv8+up03eKSUpEbWNzE7fe8Tqp0XZzZ+R4MYw69+orst100kYayk/dNQKGTdiIheI2llpD75fmsTHfcMeduHzuDJo7NU0QkS2xXvzc6+C0x7OEBov7aq60820xdGBtHGrLa7Cu24PP3jCNe97xbgyaTWxcPa/fsuecAVCR0DGuqti23lvNSpssK2lA0mudYwaaIm26r0HsXJnLB//+vxso6lAmOwT7Jhsttv4uAiJ3+lj7Z1eJRtAzMMVjldFiCK/2npzhrTOjxsEqc+axLwWHfULMKzfu+nU33+HYb1uY8Onb7lSIxpZdro+lwi6cPydIlU6aqVNbHMX10VB+jEQYioQecoSOAfjceNedWDpzFvWdHfMxvADBivt3SUu249wshB13tW6pYkvnkshh2IVrQ/YRVTjIurIEb/7692ix15bPSdjOnLHjLWNnhjDp7G3vrhRahfehWuecGF/d2EVc7DA7ETnIdHzm47+XMDgfSv34PyfmaZF0UhzPf/RmMxa4CfHSronuAj6ZvImdOGelqqPJVAdfO+A1doEWX9CrxMkaqovsZ6f63va6N2Nnh2yMLlbX1rD/4GEcPHgE7caO4mpRfns9XL50CVubm+Kgx3LwOgQ4RlI/5liJTOiHoclPdDVObXP9LTdj+dJlMWnIXo0+M+HHBIEhTvIbuWxxGq6r6NGCeZM+Cz0t2WSwM88USeMt73gPeu021pfOCjc4f+6MLbZ7/+FjKKtHAfFW3LbBDGJVqYo2kB9O5+FmNCaK45hTn/rb31EMUSyzH7j5nYb5+jmY0TpSYZLtCd5InQ7Ey7JSHCMKGL2YixkQbOw07QS/VrAzQ3p1Yg6rJxw2NcnN4vSdr8fm5roQI+5sxuF33/1GtOm5wjQQr7G8dEU7W2fZOu891DMfSrsjcHkXKIVSLqD8W4BJR05cg621DaytXFFPEiFRHFsY9TFnVnVZrloDHYxdZ6cGBbRsjeN3Y347S6SHDO5953vEe1+7fEaLfe7Mq4rVJf5+T/lI1ppAOL11d6TZMc0YZA3RrLxvfKzVa6KRz/7D7wsuDXqNUYqNVmyOWCBj9tCjzkTqG8qdGylOs7k6scZzmrb7DR5VViv8Al8AMUIlheYV6+jBqCbVzn4TVtdW1FNlbXUV3d4Q97zlbei22KbROvJz0VZXVnHl8mVRbCOc0iLpQBpXoe4oUXeF+jaBsNEJ8k2l0Wy38cd/9Ee4++7bsY+JDR8bif969miU4/6KnWoQjFwzcdG3xZJAMbN+JFMQHYnLI4Ove8f7MOh2sXLpqxLKC+fOGiHSVf04UBU5i5G/4AUOfA+F3tg2u5z34BGYtkwj9bl//OPXhF6jvp8uwRZnGjFg1NGXUpqN8yzNSVMxgSNmYZ/ouQZyZuc8ewStE+fNhpla2z1wLVpPJEkGt73uDeKNE3VaW1tDu9XHvfe9HT0S6nqsDrHFXt/YwJWLl1R/TafFMl9GJjTeuFdwqurFgJAwLyNAiAxTb8BnThaBlK44dYahu332tG8cZ2k70M/T8uOVAjnUCX0yJxae2nvjUBrqoQze+Pb3Ydjt4erFl2VzL104PypTskNndzsvhUmKbBvVeFCYAwCIsNds9Wtp0akHPv3HCZvEcbEikRF2wj5odjeAjlGHP8XGpto5SOFkyrCYBiDqFUcbSfKVMTMzoZN6vM5bu+s1xQnWYJZlwjfedieuXFkSAZF9vtge+g1vfosQNMba8fCbW1u4dO78qLOhjd+gzXhZZskmWlThcC69gI4cPOLyjCgsRy0RN36dkn3m8UYyJeLqEOZY9N1FlTfgHrlpDyvCsMZ4pC7TQXvj13Nn97B66ava0ctXlrxvmrFr4npxX9G8YiMyeRKaw9GeCNMsNIOyfqbKE6Q+88n/mZi63T2OgWzQkPgIAeiI6Wxt503HJNruND0tD9CPNLJF9ERJADY6dshaPlscGWrcvGe1+VANOFROdN0Nt+DKlcsiGjJe5K3uuvtNKp9ts10jGZnDIXY2t7C0tKTF3t0NnJTdHSV17tWRHKfxvmynh1Dy93TqZA+9twq/l9fL8NLHGyf0CGuIvqD+jCYg9j9UXYAsdhSym0hWtaQzeP1b3y2zd/XCS3LKrl694nQwW2gzpbsHxIiE4EWAHOO42tZ9RjlFrzVztFBj/cw//BFnWotkDEmLcUOiaHPU6DVtao7F+uqsMmYDxxeetczRRYg2kLHsru0O6lOoNNMXcRC7YlI/gJ1O2613vh6XLp5XcbmOccxkcdfdb7Z+afXaCPAgAHLxwsXRafajSXK0xjQNPK7AAAAgAElEQVSvh0puasxb9zg7doUgVMMR5Pw4SCP8OfBvPytr5MCS+KB22t5wncczSSgClTQCR+z8kXBwsQG84b73Soiunrf4+tKli6MTl0zQrKCB9xcnnKiemxRGH6G2Y6FDsEJj8hoSCP578B8/nNhxjP7gzh6hNx8XEgDiKpHzF2dHMakfGoEDVmd890AD4YrEF+fT4j+2prSzSEjmkzepigqj5cSk5PMl3HT6Nly8eAbNWl0IGXfg9TfdgcpkVa24wtPk37mzFYo4C3bX8x1pcn0TDiHVdnw+nMj4uxweXyA70NVACk+YasxU9zIjDIc8XtdZ2wolY0fSNHT8aAr7tKAdJX2ETeL1971P110+94IW++LF82aHw79RGOzZRvWIsYPkLTHz2ub7Sj2PHEKzmnHagFDSz//TR/ycdPPiVJ3IAckxsA5CmhTufH719GE81CiTNLbIeix3vJi14e6WpvAMWZgIo0BZmYyFDLsxOG32DTedxoWLBDi27RhmAi8Ts7jpphuxvbkyMjU8Punc2bPujVvYGBy0sFcGUY6Lnjkv2oVj7SflTwgxtL9FoY5Br6aZI4YOkmOobd4rMoYyYd7VP7xyhXBuhzWSYYJjN9yJ+YUFLJ99XkJx6dIFT8zsEkkS1xaMDKKq1Ha9JX9Cc4+bFX3v8xtRTurBf/qI5mA8WcBBy5UXROdsEpEIqZbd4Pvp8qPdYS6It0o2BIfgCr/GGV0kPASiEzF2TJCpmzghwHb88eMnFFY98MBnMD8zrf7m7V4a3/QvvxU7G1clkRScdqOJJ554VIsklE/OmSNebqujowHllTnvXZ/EBCBsXxAwKBzWsM6OUQqKFT+vfi2+ix3NlyCrSCKQNkcIzY8wGrOcRO+faioshfmD1+DosWuwfJYdKmpYY6gpLWKJFUszO1FEWDjPzbYiC/V1k7Aa0STmdmS7vcFQYA2pLz34vxJzauyhTUpt0qRu2GBdyQlzZlQ3xPeN8dQIpqhk1h0fE9rd3t4SHnVGcI/WVVnYwlDdcX/aTd6/1ezgwsWLytpkSK0Z9lBvDfHP3vcvtLPpuHCR2IjvySfI8DAVqSOYvSWnhMpNk7xgn6jY/fKmvdWlhWzWuzvUfbBrHdUd/T52EcMqdV3gSSd8U2g+PxMkujSquTZbcuq4rOixDmTKU7iLIea5M1psljqNvH47RNPGz8+Lym3FDPaKGF5++2ixw2FmOXAwSCTsX37of8lmW7Yodl4U5zP+cFBE9un/a+vanuuurvM+siXLsrk4zTMdGAghJc0Y22BjoLSZ5rl56kuf+tfkodP/oy+ZydBppkmAkkkoNrbBKdB2aOMB27JsS7Isy/iiy+l8t73XUdEM2JaOfpe9117Xb31LXYzxtLvTwR4pSR9LgEZeVpvIk5QJtIYnSxJVoAiPCgRAGTpVePBnQizc79H2pJ1+/e32zb11xtpsf3n8qF358ss+WSdIVpLteGFyvWrBs9Gx1QzLEJWYoCejJ1QnF0gDa19LpQHqjKhFJoxQa288TyHYI0pGTcI0abtzi+3Ea6+3m1f+pz14uNlu375pG68hOVhPcdqonJo1wXvt0kGTyQ1zlMRifHEtAgP/+MN3kgrhZuGHkB580V4nVu2D1nSxWD8qy8zI1O53tZh/opU2C0nPO2AFfxbJfKjG/Sc8JkA8prHvc+2Vk2dZDHn0OM342+3alSs97MgIKJ7ylAvLCU6uoJuqMgVQalnjmkZYpU2W5jGO3oyI1GY9RamedAnPKBgBlgQAYrQBrquDMNd2JofaqTNvtLWrVwiWYHrYqNVoGBZhzHmukM5OngfohMUh19f+qCAUT57ZynO/+wWRKnFociFCiJ3qRFYLtyAQwOq8k7LtG8fESlBX4QYt2u6nt5kSywXWwpBxCKrTIAeeOEnQjG1VgmeunX7zr1gQQC8TrgPM981ry4ImdfuVCYBKZgw5hC0WsIGLY3oLLbBKrqlmqZ/NiFW/p+RTAh5SWaP6ugaqmwpsu/7tqlfSpTxYmKh+qJ149S0WQkDTvbGx3hEv40gNkASzcp6AoEepYazVuvMe3XYnawc1HrTJCFdU4406pdfZbbRjYdNAUkpt63Pao0T4kvbMueIGFqpBXYstG2SmJicpFFZgrPAAMOq99FyvvfmXpKcAVQe5UnYet6t/RNVoh/9WGFeRMlrsLB7Xx+YJz8AowA9dVTun7iH37Rx6pgNFjQOmS7gV/BHWA3TiVD8Y3j7u1zeIc7vAMgVth3U92E6++jaZHzfvrfNkax9k4uJYZk1xVX6vqGrlPGBf5LDFXPR7JtV7/sN/0TmK+q07ZueAC+1eLv1dthsnAMNJ1K9tUJ5TlXJsaj6nPJ3Zi4C9Vi+YHERsR8hnnLB3rK/TFOfxe6Cu/s53ScRD4va97bb89dV27x7w5KMql7q2RiaBv7Q8g/8aAVdoOODFiU6kqFyT90LSJynwJPoeJUfOjeiD2uwxO2Wp0Y3yReDRo8x55s2ftDsr19rdzVX2d3HsYuaTs4xc0rV9/Sv2L1UwPKfEQLG6BtoEmzf5+KNfWhvY1ibD5FOZE231L3XI/8+Rfjqgh8R0OhlyukAGD3uM6TScqxVbvSdmhJKnV8HERQeGPSyJJvGhaBfCxbz1wlI7eeo1MiHTmWq7beXqdQLzMk1eWkm7O4odKXJhBomotjnAVKatV+jkUIVpSAyPFMbAjqzNkkJNbE2CeY+TyGQAMjoZuqy5W/DEVeAgwufAQjvz5l+3zdvLbXVtpd0Bu7OdUzw7ng8jq6kNSvGoh4LVfyrIWWpVb3YO8uTiuV8RSox4MN7zrPxLavIL6c5E7hoLMsKA2d9KzMffcy4XQkfaSrSpGqCYe8bOzXrII3VL5KYF6e79x+3tH/+EuC1K8nSPNB5Qgdg2fTYmQCpdXrQ96V6lEkVHHDloCWgBYMz43LGHnPGl9ClOTNS3snWKh5FnZ77dzh7Sy2Ql3tPAG8wCwbVFSARPQA4UNvPlk2fb1vptjuVYX7vFe0k51CaMsgeZQNBDMK19F+p9Cgx97TzhF8//2o19Q8fFfZcS1qnqm20Ok3SI7BcQCcDYJHrDO2itfaiGOzaGuz2ocJbgaSAAsy+pxj1+z2kSXH9j61F78y9+3DZuL8s32ttt6+vrbR1jLayZ9LzJHThvwFh40Fv2iCK8KHZ8sAEsBvnm2EBQhuTa+X719mkryc6gUcbpfcv6wCuI40n8gEGIWOOXT73RtlZvtdXby+3uxpr6203Bid8H71miADwLINQcBxFHLQ0Y2WQntKANuHbOo0w+Pvcr48a1oYq2ZSP6ifZb4nvzC0JW5gTq1CTcGDavxsg4DVBlcsaCWvUm2rusmiD935BUeLOS2O5Cte2duXbi1TNtA6dgD1TVjQD61bVbXaYZYbg2YQnqJ7UKKN5JVJcgBhCsadaxlKgpdBTIQYKZcq4SStKOEh/6AbbjIBzQ9TAZQAT5aYHSlaft+6+cbvfvrLW1G1fbPYApe11cCS4Wh+y0Yj16+jNxvN86BzJ/ZjGgzum/fPrJ+/TGe87XKiRqNb8QFYV226ouqtrdpz1mBCI2T+p1oCFHBDAECCafaUerUiRzmFjh3E7QcB1qr5w63TbXV0lnhc1GVeyOwxY9B3qzTBvhWLg/X46odsZwXyWElFoc5EGs1ZcCDXVdSrbOlxPznjCOZV4lQsgOYZydfADhzxi5USUJRPjD195o32zcabevf9XubK5zs3ELMkfVAbR+NojIE08cJeKOJU+/x7etP01BiAAvXvgNN5ujkKIyi0cH0Bq+hG5UjRpf8H2wAbFR+3PN/Ey3s2Mel2J6PVbCL17fTkw2qsezOiszNeLJ3lw7ceYNOmRomwEVFurda+urM2FXMnYUqHjLAe7vW5nkxvPtekq0L9Ze7DEDoTxoLsBtLt61aB8mobxW1G5GfDLxEu44ok1R25cX/4MfneD1bl77st0hnQgcOCFMD3pONvYmpLYH5kWwHy2SZ0a/WOJ/ijsPixIstNkXzv96mrSe0p0eG8GN1WXYQOAZzIEWIc/dL+i71RM/CgujlDjgsb6uM3bJPwe5mQpVct2Kaw2AJHFKa6+cPkuqRoyMPAjH78GDtrJyvTtMqqPbZsXw+zlzOpMAyp8Jl7KIPZal0+I0qHMC1BzklgFJkNPNwIQDaMdcuzppoImY2vSJls4ZAEccoOdefJk+wvWv/ov1akQ2nLyEWjbsL4afu0NEiS3BrWhanOaWMI5iiEJJ5eO7N/7Jxfd6R8jMD913NfqmZgvwcLoYI6ePiDnzCnbDyRWqcn96tGqB5Md1kmvHpU5zCHPTXMeOyvmF9uLLJ4hU2drc4MlGFm7l5o2OF0tdW0I3SADY2xVOb6NjcjK6SQkg0smLaAVqtzQxWoDU8eFChVU5N3TG+ZTDJg2pJoqOI2tz7cixYxza9tX//ne7ufw1JxbSbNmHSpIIDpmG2TSSDsATUIg6Uqj0j+LQGrZMDBCe8dNL70+hluSAqBdbR9Y+kRMgWNioA0gKOwVdyYEdQsNfWlajgns4ZUjTQFoWtegFzKbIRimRoahN4Q2+xEwoTTO/+FT7/kvfaxvra+yUQBsQ+LWHRrFtdMIoaVTxgkeQMJoYU4+GY1nbd6qmx6IKqKiig/B64z26AHf1OTQaPoj2KHGrylZn+Pt0Z9ouf/FF+5uf/rTduHalXfz9b9t3jj3J+QfJjDG9y5aoxmgGIEgWeTxsjvjBRDhss7b/Yx9BDt+0Tf5w+QPS1ygLlLgl+12a9N0JghoqnAJwimUze2xpG8GUnoefiUZaeCxtYkIi60Z6uqlj25O1vOm6Dv8ywdaFvftb2+21s2fb2q3raqnZ2WnLN67xwYW8CdiwJhZ1/yAyldQaoEQKMdWkCzelb6tv/AgKVE0y5EfCaEfSCy7BVP9XNXFxqOqTra7ebh988G/t5PGX2xLYEiDkOLEGIdAEGlARcGgQrorHkdUDH5oig9Tgtd6mOMPJ5oPkQlalLKCzJQeDxlE8iJ2NLRinI7ZbiyeV5nRy/xMbqhYVLXYqO/SwS3IAzxLkClUZF1D57uScITo725N2/NSr7fbNa4T34HpQ4xAOaJioZIQq1AxpKS7v5yBToQz5VTCkVJuTtJqyqCqQpA5dHUuxUth/KSldLHFKwqoejnC2JksYpcB32d0207JnDXAtlQxi+AZ1jfEW2zucQwZoFt6LnSPBCYDwxxXL6lDOL5joCKFXjZmT1sTi4SEB36WtsXTizxj8bEZ+P6FSTz06hNCNh6qUDRd0SDEkXtQUlS6Q8HeceZMwZdYXBEA/Ovn6W+3m8lVgSLlRt26taHE8CObbMoI5BTFVaEmqz68WWzk2KnP63YkBB4/aYqfPBOYMX0ySlNJjDVsxIE8lysIeGJw8b6TcNZJO0n6D37xGBLTNHALPxXArspklQDO2s0NOuHtb95iKZqOCexnhXzFE+8OnH/Bk9w2HNDlbJVumJvpsthIk+jyrRQnF0ozmPHPQL0mpjkoQZosM1TnrIOhfeDC8PPovgi6hSvToIjiNsIEnz7xF/jEAnHEfqPEsdGL5qPP4EdFYET5ojapOa7go10WFGt6fm6PWpkQuNDJOzECFIudO79ydKGSz8xcFLSFpcQiUANq24zjajqMxs+manKCnjXCR/RkEufb6EYKCkpSQMnKrqYjDeWXZbJbnAhEuD8JeLmdw6oZn07PxgiHLaWHzuGdcRp0GKEBuEoP60BbcwwID6HU9WbugJ9FZwhAE6plqEz+bbz9CL9gaxkI+pucKB024OYdp6QFmbV5NinjAePhpeNMzJKmihnvNDpFGUZSQaESCykDHTfrcLJxId7pogfU93Pewiz5xDHNAcmDI6eJ5nMPZt0BZ02WdsjXSXhJysTS5X85FFDhyqk62Ptpicuniu+JUsXwn5qZnTika5bO8XCQuajwbSu1g+yhbaT0SRKUXVQkUdW0yBjX0iPAbniAFD5wGCRI3jIYKRNdcIWgP+sGfnyAPORiI8LV8Q0R1GuCq6hKEjjPLYJON6aID4znaCZ34bwq7bDcWcjbRkky6kiEJtxiuWhBjfxlaudFR3Z9qicY6UXNgpMbhxe608eCkJ67jzmd5YeL8cfMOmDQXc1p69+hen9pbBQN/R6jKwfCXPv5N3qKoKpXWuHnGnOUEx7mQsyUvOw5RVB3SfLAb8sQ1mTYmS6xC4u5OD1QnZvP1gv4Erhz8pVWNcnQkVOP0QHvm+Re4qWBTwtfNWyukn6A3ySxWAAvyVtP7VHFawZlhpHIydTpxo5iT5E5MQ9VG4CvXe48qm0yiT5WRPemw7KwUtuOBQDEK4LFOAqn4OEVtx9xWf6mPniZ0GcIoAYxGpq2HULDEabWU2LFWpTicmV8KnZhata2m09BbXUZlDJ/FaKI0ApL7k4wOJTwxL3naUxcwjQf5ZJ9u3BEErBpBLCRIQiqGRm2+PfEn323PPvccqSTxhRInrscMAMD729tkG8LG0dPmu3gRDaiP/dVwtREbd3SttRP+LSEbBQ8+OzabuYKR/lVUEpNh6k5DruCvJFNY07Cxw0Go5ARjU+P9x//JhufgAcwoBy5Jd534oZm0T5MLH/0rq1483oVdIBs/c+xl2fqm8WYHNMwktQWcZHCNcpSEpYs5Yo5zkMqW4GhhUapDe5EqOQbtO5QJCyEhSsjWOXTDS2AMIRrjTp89S55OfA+c33BQOILJbI1KWcqRxL2hbSKgSiIp0zcSOXIKs8AAEEbFwjT1EK33sMthGrWV8W69JOq05nAexeeuTXOiaF9KF9eMNoWwc/18GPJs+TlOblXz6XaJj9A10acX3p0KYTEQFUmu0AmxPY8nrGFPQwTojZY4mZOBZtKecnIY6/qUZL7IiKPtnTvMgfCgiiU7rWIB1ZDVssp9ILcDWO9UW13RlN6Nu6tkEEJ2j+zDYPhzxSxISy2iMk4anrrN7s2kN9PrhQWiEBotk/KmzMFgYooDV52umLeo/ZiebDYrab16WMD9xdPucbK/V0NevAM2P/kJYO/w/ELhylzVCCsagDabF+bpHl2JSONFv4v1aFRRdDId4xkpCjyV0psD6Ie/0zFQykhT64o9g4MWPDeegW4ZhrK5vpzSphZ+FDUEPFTv2Cuvnmkr167y5e5uronczYkdqjE3K8ZZVNyMcBJOHGrSek+ke/GFgkpMC+7BU4TnOuAikWktYeOl9r35hjhp2BycOxs/x+3MetnJ1MFBfludKTBP7Et3eKf9MG0XES0DRcRN5vQDHM5RtIr2JC22U8JB4cSBnpz78JeKswtTLz3yvZEZktrTw0hy8AAOLQy3ibSl8Wx42cp88TTCMwTkx4uEFRmqBpkSXR+4NQmF79VhROJbSYQA7rXjp063G1e/5qJt3d8gYgVCxdKsNUV6oiPhym0btEBEKhZdqBipSxHQJ2rgOAr3VGX+p5Aoo3Ajpw68brovpBFrgPdmehmzxgszFKpcMS34LBNYKSfjul1/SqBSWuY77Gl2N67fSXNc3NFUxZiWcXhpsy9+/B6LnWH94xksqqOnMp33jqOGFB4+BqaeWdugGVgKbVBnvt+WOO9aJzfM/iwPTveYhMClU8+G972I4kSHEkNbiJlQEjq0x/bOtJ0+c7bdurHMzQH98vr6Gm12TwyRqQnZJRHEQjUne8dqUkh7Jgca5lknjGKumc6oHDe0KjOGR1vSA00TTn93PO+0HkOYMVtLGyikqPyA0e0Slatr6oTCvMmpVVwvhKlgVPiKiYRgwy/Suks4a7TUEy5WL9xoCEnd7NjQ/FCGXW4lZAWSGbUGT5eDUuz49MDeN8DpTBtwVEzKopmDOUhwR4GCqp+w370+sD2AgIAIEepx8+cW2osv/Vm7uyZ2QHCRX7++zDHInNG5s026aPGaisRWeX45atgcYsvIqCBHM0PQsanyDVwx8nShhGVDaOVgIfqginU+H825+uwBhoP4PLBkAQlkrSEQ2fCUhKN2c/BynWQy8X1om5rBjOfdVbYrez22Z+jFk63TkpvGkajA9rSuYlIffh7JlIqEIKiYEs8RN+8xcWcDVp4Ym4CXxwMDyYm5GrhGkitwsLiAbmLTiXHNuKMolZR55pnnid7cxcjG7Yft9q1bYmBIWLgLFWlqjU5eo9HJQXsQLmQikRAJcBNcIOEkQA+HBSgCwgh4b4bajd5ybW6yWlgLCCiETHkJYMWlIdI8iaQLGvmjqnFtrgNO9UzBTodOZkbTCuTfKIGEZ4BpwM+zrvHQuwBks2OL8+ewJw6H7IFCF3Ni3WGoZn2JamR4h5HIJF6wcHHgEo7lMwT68T/E0wovSKVpcLwkVlkraJP8nDXi6bQdXnq6PX3saRK9ovEdDhoHssGjNEpDmkWxKE6HpuSJ7opwXla0RPADqUtrUJxJOnT22IMQSVO9FlKsSAk3Ewfn5NHj3xZB3UxBCNqyF5ZS6gUEWQPl2CJtxAvuo9hfMXRYDpPLx/tRU1mYoE0gBKHepM934fy7PY5KPJYTJifdRZJCCSkPO2KnP6v6CF1HBCcaItAibeDwvOvvihpT6UyoRhVCNB4i92WSBO2rjx+3g4eOtGf/9Fm2Au3ubLfVdbQEyfFDEoV14eku2RHiiCoxInADrquKuatXCBMJbHQPd6g4IVydiK5kt6zm5YXvtsXDmlVK/8CtuVgH2VRdm3l+1w5U+VPuQRnFsZZsP8JweAsl1gyjkbG+bFAwVGvUuZXNSddJNDQTM0hqZbOTcYlKr3ajH+GGmRaa5BrpRYkwdk1ORkhsArcdUJ44cvlcEgVJFQZUgJ9jQznv2qMaBpOCFTrGP8LxObjQXnjuhba6uiLmgqt/5IJT4OLFp5l9H/BwRssYANE99vCrOvkD3nD9TJtBzWGzpbDQwm+kT0LKqNfkGhA2xbGSI6vWXmUItykETASlrm6wJwWyx+HGFITN2Y2QMHS91h60ivMkPGBffPbvU0gWbqzyn9R0Xjqbig2A5xwg/0gc2GlzrjdqpSaEEuPGS8y196dgByugVGPgSLGjSSRQLbtmjVLn8eMnCDaEqn3n5//UfvjS8/LaCb5YEG2XB7+HmUGU13a+vE9Y8NFtOcq+FE6nP4n/DkOzt5hajuXLAtLs3RwqCPW0rFOyma3dq2k6QqpVu7ukE81mMJo1BIkPWKNSviH7ldw6NWlICwsMmg5aJDXNbPhw3H1me6aN9ihtMREAOQAmijfAQGHUKEAkNSoEptCQ+BPCFQdCp1d4ctko3XMmGgj0Ju01ZleEnf/nd95pZ86cbv/4Dz9rf/93f9sWD8+3xUOLnB8GbxueNuNSsCog/jVlCEMbb3TQKR0IWPq7uA1u8Y0GDL02n7Hi0p0jTZMFO1fpvLoNyZzobAVWQbiXJ5N3p6oHHYjbh2nWDJcCQzPeGeu4uLRkLZsSrBy43vi/73RPLl14b1pZimJ/ZZMVf2MjOLBlH8mNPlP6hVPJ8bG+u3G3PfX0U7LplHrFhUlyKMQTLzgkP6paDs8YDRmTEuHA1VSSVC/1Y87sRBPhw3ZwihLnNz7JiIkftKUlTNgB7xlCL/V7YeKuSAKM9nSbrwo26ekOl5uydez88OmjlvJ7xjbG58m/eZ0219bW1zgkhtqFhRiphK6u4/OUHEc1p3aKmJRK0Yoh3aNHjCggvNG0iumFQuUhKpypk0sX3p9ubm4yoTCcrlrBksUeIL0JHSV41wn6ZcNjmwPzGaBD2ShVYSCRrF512g6hNdNWo8+FL3WEY0m8xF/garFeiGQDxiIjiy3BTCZqfjIhXgsoEKxv4lRQXfPkmesFz/fNN1vMpYcbpfssLKjITmcqQA6CwBpKM6eDJQjcVEa6s1vmqGSjKRRutpDGEeZOTJFpNRoeU54pthtTgZL8GTBuJ19szyM0vBc2OxL57U6ZbiZ77hFNpeEbkqVwJCeieucSfgLj+u8rohWFpuJu5ZI9ycBCoSyXwQ8u0EcYR5Sga89hlBHnj+gLagxOk3LvimnxBRN3//5WO3xoUaB7xPHz8+3QPOLgbaVQd7XoOAAYldSnHIw17/6M1kOFHsKDwEQcjHotItG+ptgj4j/AhHDqMMeD/kkn1TPmb6YWoG5PxuNYN8dPoAUPlmCsDZ5JPDShCoFJo4N2+ZPf9s3GpmdTojKrg5bNrp57PNrYOth2Zc6GdqAtBidocN8Zv5S5GS44xGEj1bJDF9zTfaSdB1Q+geJ7OVomk7U9xKhGxZdqm03SvWYI8bzppWIee6IRj/MW3m67HSaBxTDpzhyO8RwqicYBlUPmvHRYD0ImaEh2h3V11gph/ygwKI6Y3A4nPp8VocCgueRmylPrzA7adIV9cFjjNPJk/8fl302JPCzzr5SEGHTGRajlWboPORs9q/5lnxlzLqonKaceJy1pPZ40Oyg1BOLfozatQUgQU8hsc7+Mn8pmRwPd37rfjhw9qkEpHuGgbNkA62Xj6Yi6GY+x+67CIWwe1b5LuECSJgYGGPLOnY127Nix/2f6IgjQz2n4i9qWdhnVO4aedvwQdiE7FzPFOFzODu8xYGI2qRMBMzmG8cA8w9T8Lip5iXhkFg4wvp98eumDGXxCbHNOeAXwRwhy2hmse2J8atjZCHnYvU6mGZmeZ8Eih73zOEP99+yJ8h7FAcLCQ+UlYpAfIMHqwuZ5liNe1/35Lv4c1X3meblJT8+g08HMFNbYyBPlx3MPwZ8hCIFSJSunRFBoJvX5/VqxC2k89jIlKbZ1HAZBmxSDay112jXgHZ+7t7nJwg5VPFuD9sQV68YFnHx8v5c6ocbjIWsBRzEdL5qXIpDPbSfDSYqNnG2pqfYDf8c1qhbQQBi03oxMnDzYQTyjQHH4CBRyjDGiFtImI5SS1BvAaK4xLBJ6v2BSxvuMal7i+TwTFjNdILDdMDlhJkz7boQ6WMpJKI8AAAdhSURBVHeFTPM9/Rqn7SGm2TLZokWOZ87nJ3wJFTxtWl2TCMY4SHD8nO9wf7g6QhVbU70/gokKBbj8VZk1NxaWfAk1xOXLv5/SPhtaEw6x2G+l8gZTQiQvdrtWYvAgyYpF3UeAcpry0hEYwXoH9kzJj9mxilGfta0X8SbOrainFL5xRkhaVL0IQbf0Re8/l6DqkMlOjAVPn5g1aY+5NQmIGss4M5qJEPO5g0MaT8UTrB9ULNYFEUzleckzVXufE571iTnVeqpfLHYYzI442VwXLazv6VYuv2tMwOSzzz7iZsvDEyYq3mtuPLJiY6pMNjvqvnrrWqJxklIQiGpXCJbWnrGxuSayXimPytFTokYxcwowOfXwgBH/Aq9u4rze751JQGFuHAmfoDxiampdOUmdYQORFxdiFT8TJaZBfGFWNudKjbBy7RD+5tBwhBRNgRJSWQtBqPT90cwY7nIsqPP5ps0A4RBKuHpOTQfsozhKQ2OHlGGz8eHqqWbzUz8epzykqFC5QY1kY7Upo+gxWoaG/R/9xFGvtQ5bncR45ji5meKjk5ci/igYxPGSWgRXqVOdTswM4cvfIoiBGAffpsORcIr3Mxl+/02364hFQdGLBFuqM4DGrBlMFd5V5rACE3WvmkmMd5/3UM1cdfZ68GifbVblAMuRC0NEogL+jgs+9Ds+//xc51SpH0p5MKiObE6kKDndqp5rPbyq8bHE+lskOLadoUahg8qmj2sPxCfGIIhZUClQePxaCBPjwvbbYQmNNq6TGrJSkE7d+lQmWRLnbzhW0tUiBxi5+pz4qn6x2XHWlMMPBNgJmd4TDm4ZIV5qwTo2/969LQpGZ2xy/h73TBkzZgIags7XnCpd1T/oG02NZ8QrNjtSk1NWN50pOvdJMzXKAWUhtk0hAY1pGBAumqmqKbJww2kbZdMqEJHq2PiYAZkQJVeGV6xTgRQu0SX2/BGC4GVUsx5hTH+GjGvEe6BZgfPHFCb2cMvJnzwP/qQ69vgFePO5djZoqOtBWJDTCUEJiie16W9zziJAua+c2j2GeEAE6T2Vas7BgBMatNDsgTKYz45sYvfJF1+cFw9anddRSlYjoaHm+AhGbJaVeMc/V6ejhh9V6rT4aQ0a6jhCNpw6lDrdb+wifjYuzxsBVSZPSQdWoAwqYJxpZ4mkcalU5cSYKuvBw4fUEuRutIOVEI4LzchE+Paoea/GjI8Th2q/TzLUveJkkcQP9RxBzmZn8/P9CBQg1keOLLloFKbkUaHTvjjTZh5Xric88//8XDZbLrw+GDWkgsUgcmNhxMWOvExV9yqciAqK0GSX2YT+UP6bed2OIEHixm1GrhvHo8c1hkerNtZasKnhHTZDi2xwIBGv0DI6BQinDh9eGsCA7n8Hj65wCM+IpEo2O2iQnETew5oDahYLOBoAM21wIGarxqwaLhmxmouoMbjWAKp+ND5mPaJpIgSgBHvyyaOMtSHJ/YAZCxw7zh1WnA0vT433mT2ZBIqw0XoBVprc+hNtkOZb/Vt56H5Dj3msKoZ22JmsEepI3qr5iGceCR8/F2xoVqWbu6yGHkUooRJRi0fOLoBJBR8WPlflWBErPK54huQa8g7yA8yYmNGI1hJxxMhs6CRLTqScqoH/jg+E90h0UgWY4bCLRtV5zufzp1S6+VFNeAAPPbTfSSbxmZFBq55xJEc4LcGH5GVrI0EAQ8fEpzbSmbId1zDcV2bQtVfWwQL5d+gngCiJk7V/w7UnmQ44xk50zeLwUvH0MDNYhEMkiEOodJA0mouHl8hJokze6GGTf+DZIrPGr2cBq9kQkFBCzejezmWEPJue39H1k6cfEYUEwKEVhxBopHUEJEIg1a4GSp1wMSly0KyjBX7fh4BTfQEgdXMh9hICMJMujWRp4VVPjuufF+nqPjXYzgIgz5WntcTY+G74TmP0qTWcqWMt24akdk7GpkvCR9twTnwWJPY/mw2nJeqf82bNTMgcOMuhYBnU6GcszsEF0UzVzc6192ukaBeZORMRWJtFSCMEw2fQy+XfEhTXsn0N2nN7/DtZF/8shy+Ck/tqr9CSrGIINS8STNCsPjwo+vJQhEwAanxspLzrYMJif+Nc4PuCz6rmTKkMrpr5ZJUsuTlWCTOJd6vW1H5xX5QZM1YqKjtOVcITLeAgxgkvSxy54cmbiNbsDTwnlPgQ9nlSoPlX8axy2NCgGF6xkf2iBpvF8/YTHRUPXtCcQDx3nLrYeTbulRFMSHAwDGQXrUqwOKXEoO3stKWjRzsQQSHfWMH8HUxK7D1zFm/A39y9KenyaGlV3Kmlocbria6OQiS7OkuxPbKD8F71QJ1+0r9E25yGP6u8uvFU/24zDYlrdVjiE6g47+S+a+PDdAxgdU5U7CliWXB2Yqgc4LoLwHujros6d6V4dmGB7feO1SNssPOY5Y2vsXnjpPJeU+H3EhYpATL4YhB/R4j7oeImSVvBK4eNX1wQ5psACg+hjQboPlCiJm72nAbYl0oe7TS+7/73fRjI9n85OQ8T7wFtAwAAAABJRU5ErkJggg=="/>
+        <xdr:cNvPr id="20" name="AutoShape 14" descr="data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAHsAAACkCAYAAAC3r1GFAAAgAElEQVR4Xmy9B5Sl2VUe+t0c6t7KVZ3TdPfM9ISePIqDRhqhZAn8DMu8hXnPmGXAawHCZDDmwUMYk0GABcY2wQSBSBaSQBKDNJpRGk3OQTOdu7q6ctXN8X/r+/bet+7o+fbqVene/z//Ofvs8O1v75P6ylfuTwaDATKZHDKZDIbDIdLpNHK5HJIkQSqVQqFQ0Fe++Du+n7/j116vh1KppM91u11kUmn0ul1ks1lUqlV0Ox19bjAcYjgcAAkwTPi9XYfXKxaLun7cm+/n/XuDvq7fbbfR6/X1Pl4jneZYEiCd1ec5Xv7ni9eIMfIavC7vw1fcg99zrNlMBvVaDYP+ABOVCjqdDiYnJ7G+vo7+cICpqSmUy2Vdj/95bSRpNJoN/Y3XHQx6+prLZFGv11CpVHQvpNN6P+eB9+X99Cz+lXPG8fErr93v9/X+mAP+rt1u6/7xe36en4n38JHHfx4MbL1qtZq+JgO7ZjabQbFYQurRRz+TJACyvtgcDC/A/5zAmKj4ykXW4g046fZ3CklMLNcAyVDvyWSymkDekO/JZCgIPc46uFx68H6fP6JSqaLZbCCTztjkcuFgg09RQAYDDJNE10mlbHIyubx+jjHwPrwff8eJiYnm2PL5/GjSY3K5yFxwjovCx89SkPj+drercU9MTIwm2+YgrbEUikXdo9Np6bq9Dt8/0PizuSz6w+FIiDlPMU6TBKDVauna/Bs/z+cZF8zYWHr+VErvp4A1Gg1sbW3pd5VK2TadhDBBqWRj5TU5tkzKNif/a30eeeSzCW9EqaBUhzRmMiaNsWt5gZAwDoSf4QXGX3wgTjDfpwE2GppkLn08kIQ+AbLSHKYN4sFarbYmm/fkq8MBZzJoN1vo8/tsVg+RzmYwMzOja8YYOAl8qPHdHRPJa8Ru5vslKJkMEkp9xrQDBW44sPFo0pEaCXOz0USn28G+ffuktXRPLnCvp89QSMoTpp14T16f8xC7lb/jz3x/aAj+HEKgsQ+GWshWp439+/ePtGyMnfcZ9Hsab284sE3A3ZskyOZMI+dzuxsxFlnP0uuaUHGxbQdkkMvGg6eQplhwx2ezI9XDwYeKp3qhpPPv8Qq1rxtQLfUHSHH3+04P6YWEwXYIP8Ndwr/x//b2ttTOxEQF2byZEk5Es9mUFOt+aVPNMRG8X71eH/0cE8txUfXHK8yGFjpJkKdK5GK128hkM0hzTLwfhaBQ1L34GalvQIuhuTIjos/SJHXaHZTKBY2fgspdSIEYN4tUrRT8MIn8Wwidmb8U2u0OUukU8oXCyByFidI4+n3kc3kMYLs1TClNCe/ZbpugmrkbjjZNMZ8zIX7mmYcT7hqqU74K+bzZwIxJTbw4UP6ev6OEUgVJsoecexOOUCGyYbk8qKz5no3NdQ2CExFmQjug29X1ymWqnwES3xm0vnpwV/cxCqp1jqPX7vBxkc3nJQSctGq1OhrruI2L3c3J54Rwgig81CBSdy5wOZoPJBgkplI5YVxYCdtwiKYvYJg3PsfOzo7uqUV0/6DdbWsecrmChIjCzvmlLdd8pmyhzBylpJK5cfjM3ADtTlv+QzzDxsbGSHiq5Qn9jf7EuGngfIdW4XxwLkJ1x9+kbb/ylQeSMp0E38X8pe1YU9vhjPHBeSHZJ19sk54JORJUg8WiSbfZNu6+oSai26V6tuuFitNuGZrTw50sByudNtua0KY1sb21je2dHZSKRRw6dAirG+taBNpH2ihKeKjDuG44llxYTmjsjBi33i/NQ7tb0PWnJie1O+kzFMsVrK+tI1/IY35+fuRvxFyMa69mo4Ecn6/T0Rj17IlNfKfTs53X72sjcY6pwQqFnNQ+BWVlZUXjp/ks5vJaAy4kf8c55e/54nzKbGbMNNCMhXaKv8VGDBPKcfLznA9qPdnsxx57KOGH292+VEkpbxKdSnEf8UY2aDpwox3mNjkmOLzyojsLcsiovodDPSQH1u31sLW5qZv2B2aLudgUECrJGKQW39XpoD+UWjOv1zx/Si2FiLuF+jSdzqDb77k3PpQnigGwuGcR9Tq95kk5W/Ja+wOZjjTv7d5uJksHic5kHu1WC8ikJQx93y0lqdTE7pGixkvrs7LJYcYonM0mVldXUCwUtfuSlO14037uZfNGqZTsLn0AzpG0B4Bex7QOhY8CxMXms/Kz1CKT1arMDl+r6+t6Xr4nbDMFM3yEiFBC8MOZTj355BcTqhpkslJFGdDB4ETa0vZ6HQ2aaom2iu/lhHJgfJBQY1IX3M30SD2Ei5Aq7DE93xAgqTEP7ai+5Xi5d08JplXs9xP5EXxY7cApk9R+zx2gQR/JMNEC8R5JYiGWpCexHVEsFTHw8IxmI5fNabHtfnwiap8ChoNEO3B9Y10LMj83p5+7rbZMVofOkdtwOUU+rjATw56ZQfkrFNi8LUy300V/0Nd9ad/Hwz9+Nmx4q1GX2s8Vzcni83CMVPGcf96v1WhKC4bDG+8L7ztsdcyjaVWLKjS2Z198IqFNkgT1uihkcpK8YWKhQKgLTjofIn7mLih76KAwhwvsNl5T6HFpSLWkjB6jS608U9nOtNSSpLvXe02IRBulsML/ZuaFXrTZPE6IHoKeJr33rsX0nFhei3aWO4LPxWeKUIy7k2q81W5pJ4a3TO3DBdGOTZuqDDVqiwp0JVR2fwvV0nouhYa01VzU4RCFcmm0q/nMNCvhryhUpUD7HAlTGPakbrm4IQAjjZBOj6KWcDLNL8iNsIoILWOueL/Qlvydnv2p5x4RqFIulc1uwzzbcqkgCTdny8IVOSeuiqhCQqJ4oXBcQm3JexwMMOngQ3jo3FUCWuiM0V9JpxRiUUVxYSOc4PWnJyfNi4Q5TXpQJCjkC/LaeX8+JD1pxrdcKKp4TmIsFEO8drulxZVJoK2mk0YB6nYNtODOd+eQO1iefio9MkXUAAp5ej20uh19nhM5HkoVsjkJlRwlmqGUCW84TvGZiGBoMrtde26Fn7Is5vxyTOHAUaD47KGyuXBzc3OvCWUjnAuVH+qb742/6XpPP/eogkw5LcMBCrk8mrU6si6hqbQF5IWCxb5STZykUsnCKk4Mna9koAGN7ARBAvfeIzzjoLk4dPT4PqpIDmK7XhvFvfzM7MwMWu32KKzLc6L7nDhDybiLqRppTkpFQ6K0A4e07ebwaVe4g8j7Npst/Z0mioJRqVb0lYLNC3KHc2KlGt1eT9BLdmSO9+ecMIwUltDrax6klRJaDQN6KMC8Hk0HJYoCxleYNOogaaFOR5+nNy6zZ2/D/PzsSKOG4JvDa6/xWJ6fD78gMA5uAqGh6YzubethplWLzZ2hsCABOq02qpWKSSehR/q83ClpAwG4GNyx3DGx66QmcqZqAjyhMNTq9dd486PY1uFBugU0B4VSUXZ0HC0at4+h8kIoQ7VucXfT4XEAQ0JZNGiXoZs8dtdMXCyzm4kBNPTUM1TBpgWIehEmrUwY3KmFpOYo5PUzr5dn3I+UaRIHXei48aXQldfu9qShKFjTMzOjiGZkN31M1BS8PwEbLUqhgEa9gYmKhad8hWoObcnn5FgVkfR6Ei5uHL4/5t6wCEMWBU7Rdxmak5h66tnHkoBAOVmUODpOmXQKDC3MVqX1gFT18pZztDe2k/h3gg0UgMCF+X6qND68QhXChfLOzRSYM2UOoL6nL0CwJLHYnrY2Yn/6CozZOdGESTWRdK40Jj68LZjtPBfIlMW2HCvtOHetoNax8E82t0sVaVJvCF0GRPEYslBI+FwMnbhr+ZwUBMW57plzgTkHfF5BpA558rliXqYqVY2NWobCymcNDcdn1Wd890tTMqZniOvQzfT0tASJG5DzEoJuzrAJGsdvttxQtRBwrolpV4tkUi+8/IwjaLsgCgdEEF0OBBfL1Qe9VvNg9QtHwMzrJfTJRaEKlQfoi0nEZ2NzwxElG8y41MbgLTGRlwoM3Jzf2QLaAyREy2lfAallhm2cVH7WJm4gf0A+RD6vhSKerJ3q3jd3KLUBF1DXSlnSRzsjbQ6p7bAKehJYe1ZeK9RqxNpyHtMGJnEX8sXvhTJms2hw0YQZ0GegYAwVj4dQclEnpyYtOeTTyvFwiiLMpRAqWnL7G5uEfku9sTNyOu3vKdn78MCZhyBIQ8xEavyZF59OtIiZFPIZokwNvbndaqBcKGEw6KPoWLW8c0mK2Sg+kOBFd3CUpZmYGDkFFBpqCmZcwqYp5u6YrZH5cODGMjp5CY2841xOmoVj4TWofQK14wSGdqA24WfDWYoIIkIcU30ptDud0b1kagbEx7N6BoEghCzTad2Ln+H9+BniCwZYDLBTq7lQM2IxRDGik1TWsk0Ubl6bfoZ2snvcMZ4AP8zh7KM6NWXJIvoXBT4/zUxfmkJ+1MCwBjqTvP7U9PTImTREzoQtwmD+bmS6uhQUcxilgV4++5KEiCBARmrUEBxmcxT0p2jPbUcRXOC2swU39IuCwt9x0gjtlcplhWHh2PDGdQL8zaYGPlGZ0OcD2aIzxJ/lpPCaA3P0qpOTI7+B15eEc9CDvsKi8GojpjR1Y1omJpYIFe0bNUCn05ZfEF5xqG6ZBU9cUBtQi0i1e+aI9k8qME3YNJGGKJWKSIa2kLy/wKVCVosRjlK/w4wefYMsCDYF3Mz3M2oggra1tY2Oe/Czs7MygxGXB6bPZxF27iqeP0sQ220JFneurunp1LDdYSIVy1PLyWY//1TCC+RyWYM23bGhyrTQimogh/Qw0c7iwwp6c4mykMrsnh6eNtRVeG1nR6B+2DA+CCVND5LQqelJYmWvlRk1eJYf53hGgMWQKnoXiTJNZHlzLmAAGgrhaNv1ecPCeT8JL737HLFuy3QxxuZX/p2LaGAPowWOlwtroVOnZ37G0L3xiCzCpvO5OW+0n51O10wLkbY0Q7WugKq+A1S6n4dk/IZhF6OOgKQjvOQut8RMSiqcY+dzxqbgnEYoK83nDhqvR/vOr1wzCgId5Ugppx596pEk0Cthub2+FpXOkGDPrCUMUkyMM1HiMabCINlXUyN0lCSBvnDcoRQMOkemWgwjpvetzJDwdMavGUkdFzqIArHLLRwkNErEzAAOLgr/zpBJpoC73L3rVqcjIeHc8p7joQntI69BoRHSlBhAxPHH/ahOI1mTTpl2IronGzow7TaO7UcsbOrUEibUVFqklAMy/S7o4kWem8/ATcB5irCJX/lZjpfzwu8j8rFM3FDzzh0aYaG0WJ+hZl/+CZ+DIhs+Q2g5aVHOMX2OrzzxsBabEs3kAzOblvUpyIYw7JG7z90c6kJwqKl0hWeesjTPkHivQYMCMnyyeE3loxXSEK60XTk+6GBtmP9HreK5Y4kZUKvtaLG1kxxk4b1MJXeVaJAQuoaIxRMY4lkrM0kWr3Lx5StwEvs9MK6mA0cVST/DQk8TLu2uMUcp1HVMrrJ2SSJvXlEKIxJh8gyxnGDhmTV+Vo6TmxXZW0LGLoiBuMnhYx6AGEOwcTx219iYMWQmMaITwsaDwUhg+RwCv3zTpB5+/MsiL5hX20POSQv5vDkuXGzFa2RtkHLjoRQnmw+hz7ojQlvHvSc141SkwMM5cE4Y6UWUQEocU5sUsJBCxdF8KAdPtOMUqlhYRc1gnrQtgMXLWak8MyW0nwNPF+6SLwK8oE2kAIQTQ01C28nPa/cS5iyUNEFcAD53eODhcYd9DHAj7DavG3FxhEImtDaO8C3CxDUaNWmY0A5M1hAj4M90TCm4XGgKJ0OucAYDIg0oVQAPYWeaNUfslDhyUItaMfyY1GNPP+pMFYt9mSDnhxrNuhaYzgWlqpwv6uE5iAjutbPH+Gjc7bSLyiyNATDSAo6XCzcfZc2C/ODok1N0LMzi5Nv1OB6OY2enprw3BaxQKJoal49AEoGBJYwciGLxPZxkqr+AGyNRMA7YRMxLdWjYQErXpSaIxYisGxcu8PtwgGKxKbTB6qGm0AJ4WBhUKQoRx8+IhQIsP4SIH59xLEbnNRk2hRMs6Nk1JXludHjDBNIp5Pt4T3EISH4grE2giBh8Pi9TKij3iWceSyg5TGVyMFnu7I57fz2qtJYgSdocTly+UEK5zLQl1bqF/nzI0A6GsBm5kDtcUF/CHWuYeAAInHCCFoa42a6MGNESFvQwzQwo/CAE6ULEh+N/20H8m/JAcro0CQRcGC83GqOxxU4Nr5XPKgH0JBCvx8WlL6A42Yl9kXjg89GX4c+2aJaIiMWmg8YF4hgopAzBNzc3R7loOYtyuIxXJ6zdSYYUNGooJm20OMp7M09uiKRsuzuIyk0QtMmksbOzbSEI4+uJsogYEcJFXB+OM7GD1Jce/aJsNrHtGj88HEjd5tMJup22EvrJYIB8sYRSqYzSxASq1UmUJ6Y8xKKDYyqf6pA340LRVlG1cuI6XebELbnP0IYTJKTO0Z7AfkfeKBGxXneESAkJC9za0TeaAJoMjr3bY5zqSBi/IoASU9nKjrmpUa7aKVAUXu7+yJ5xYiIk5ELyvzYA05m9rjhoy8vLyGWY5m3ImYpEBdOvBw7st3yBzBnnxeJ2vm9udlZ+TrNFUqUJI22tOZ4MpxjimQOby+cUVnEHVzwCoqqTQJaK0mB8z6WLF0zbFkpm5sjedSda8+Kw68hmf/mxLyX8ZaO+g067jmGvIyZIPmcTORx0iOojRQaGXPoicoUiKlML8gRJdqA0kiJEOHUwNFQqGCfaCV1yy7bk/Fy4cAGLiwvYs2ePecEOH9KeinjgryAdctdzh8euNrtkSX9OEAkKVOMUDl6P/zlew9oTQY8kSWSFtqVQKhSxtramu3CMAUhEJDCeOQo1zK9rq1c02advuwOf/Ohf49a73iCHs9M2XDoyf+F/MKdgmT9T54pcHCfgV+IOnLdxti43bbtlISIXmxrXHEFuImozmxyxiJIEa2uGIzBvwfmi3S+VLWFFTaJMpUgWBqumHvzS5xLyoNu1bQx6bXQb22g2ami36yCLI5fLmFpk4l057RQq1UkgW/IwKytUh7TeoiQsh3K5guGgj1azhYcffhhveet9MgecUE4+NYFiWIVK3EGkPNmDmUNkHjOFicTDRsPIhJxsqubAyvk3OljdbkdmCJ6WLOSpRSioxptmOElSgBZ0OJR65cQyAgmTwPtywng92UDPpIWD1WvXsLm5gTe+5W34o9/7EN7zDd+MhESO7Z0RHsAJDQHu9Q13N66bRR1yNDNmvgwhsx1Oc2eQr+EMNJvUKPSsFW45Pp9JG75BU8DfUROb+bHsXIZhpwSKiaqszKbRr90UfvTjf5Vk0n3UNtfQbzfQbTN+LYgmw1evb+nMtHO4h4yrBZ4QB88jTbJDvojiRAXF4gRKpYoGJL5VviDItdHpeVrTmBOBo9PmcMEIhHCSRdFxZC5if+4+Tg7NQLvbcWpSRfE3QyXa2Ga9qc9ZmJdCtcpkRV8U2vg9J4PcdArG1tamcHZOEjNh/EwQB8JciF3rW4mfbTS2UdvewA03344/+59/gG/51n+jzygJJC/egB7aawpKs1l/zZgsvcp8g6U9RcaUo2lzIoFwX4S7lbtaCaLQViOMwVk5bhKEySeGFWTyTEUXTJspbBsI8qVzq4TLX/zZf0u2tlfRqW9idqqCen1Hu6TXG2gnKF/NZEQkDpwJkmT5YMwDTyBfKiNXKCObLSCdLSKTy6BanRKVaXpyGps7dUPcFN7Q4zfHy0APc3I4mIhZd4n+fVQqEyIMcFE2tjZx9uxZLC0tKQ/Mscnm0oZlcyjm8zh27BiOHz+O6ekZdFpG/Y3EA2Nnzjb9kJ3ajpH0U4aARXjEcZjGsR3HCadz1GzsYGdzDdfdeCv++i/+DN/2r79LGiLoxeMevj1P1xiwYv0MtYvDJ1EWjQkPX/TAsoMsEk5faDja+OAO0P5qw4CgEfPvpEQXjXiS92oRYhTOy6P/QPuukPnDf/rBBANOWBubqysoTzhJYWjlJ5Q8euIcSHjc4chIEDI5qZpMtoBMlra7gHxxQna9Wp3GxOQCElJkCcP6i+GdqjGodpBCd2ATzAdReU82JwDlxZdewksvvYS1jTX9vecxcuzWcOzGVfHoHtz5JUYPBczPzOL06dO44/Y7BOoEZYcLFHbbgKTirsOWSrQjDB2DdnV9Yw2HT1yPhz57P97xvm82E0LOuUyMOUfhW9Cho8Mlm8xQivj5iPtmi8fn5e/DmVVenqZnQAEzDrrSlA6bCqyhqePadNoCkoQRgMCNcpNmNpywqSSVo2rSJb/xKz+eFLLMTfeRY/oysbonVmGYnbGgPC5CO0Q3n1IXjpI8cd0ASOdyUunZXBmV6iwW9h7FEAa+iKtFe0ywwGNvARwYKmy5cPkSnnnmGZw5c0YL0uoZm4NaRQ/ioVKABLHYoeqCIBDhEgkVfHCKFBedCRSmGMnEvOmmm6QFIg7ns0Y+X0BFwsXxWjKyaTZWsbp0Ea+756347D9+Cm++712iRtEfMNNjfLjIm9PTjjy9tJrnlhU1EATSHBAM4WLtEhW5Uw1MIQ/Acp00WSJe+m4NoCSfI9RMoqcnnpwzyKRPVI44XGj3+LX//P0JbVKxVECKnGXmdJkA8cUhmCV97xmeqMXiLjCuuZH7hCwxFOoPMTk5jUw6j/LUDKbnDmFyZlG5XQoMUbrI1jIuZCjz4osv4oXnn8dOoy5HLZIe8mYdirUFNI6a0Qu5YUzqRy/BmYwc7DchFBa3GzrHF8fBsIg7l/7I1NQ0bjx1CqdvuUVJlYjh47r83M72GlYvncPb3/3PcP+n78edb7pXBX6tesMWeWglReZMmXOpHcl/TvlSalh+gKlxIYb8zMDoTBEi8omocZjgiKcbkFYfxZBD80+4QfVMJC24phDsyhwFMQg3vYFmpn7xA9+TCIhPBihmWQJEN9/LdrSjzdBzNxIrV/VleIeUfDkkeaRdBXECaZyZCJia24NuUsSpW+6SNy4MmA816GNlZRVffvQrePXVV9Go1XVN2mYLxQzgtwW1laMW4WLzRS1iEmsPPVLd/n6S+cY/GzYw3isChvLmNE/GvEwPWVxYwVS1iltuuQWnTp0aZfc4ofXaOlYvnsPdb/46vPLyqzh2/U2y2TQtlrbkeI3kwBeflTl5YeacI3rVjoFHrK9lF2c9IyxD8XmAJq6OhRYWC2hRZauuwoTF5sTSzj4tUtkULoOxeyq62N3ZKaR+6QPflyhWywJDJh6YRRrS1hhFKQj7uyGRTbAyQp7jNpaG2fRR2pDFe4UK0vkqbr37rQIWRLYf9PHZBx/AU089iWa9MWJNWrxrFZ0Kl9xWxWLbw9kuEanPvW89rDMzYzEJqkilxxZ3Idjd2TZ2qVenKvNnyzkbIsg5IaBx04034fbbb8fO6hWsLl3AqZtvQa5YRaFcVdIj8TqrkTlIGS1bfgSdUa6E72gOWz7JWHgU8KuhjtSNxgW0/IFlBM2AkZJlSBsdM1HFXJOEuFui1lBN2/l0DFmk6MLxyz/3/oQDK5XzSDn91x6YWbCWFps7ke+PhAM/Ssg0dlxUUHCHh0dN9d5Psjh7cQXf9h3fJ/L9o08/g8cefwxXl68YgDJWSx1o2jh8GQscO9cEjjvbfIRQ7UNpZ+On0QSxIsScGtMMAlrGXiEUIUghWJaZM3iSU6a8fS6DifIEKqUK9i/M4NSNN+PW2+8UM1aOnlivu4wUwqaMDOhAEZMWS5Z2WaQI2wzyNZzRqw3j5BAurmWwGN6akFD70L5TG3EjjFBGpmhJn/Y5ZMREDSyOn7Sikys4D4Fs/uSP/9ukpKJwMk4oUgPk6FJ5WQztIyU0EhvipzG0cIaJr7iQLKnYtNVqK8eayeHVy1t45zf+n/jkpz+F8+cuaCe3O1TpVpyuHUYO1oi44EkT7TjPJXsFRnjd8uG1K6nGBhh4sZyx12yhtcjK8VqJsNlHI7jF38eFaFybjAtHwKb58gQI1jA+J4tmfmYex6+5BtccPmDeL3qkfouuJIFNzLHV7vTiwVjgKPYzgQzv2ahFgmY7lsAJuJNzTY89dr9COdaBZ4NGxXsa8ZGOXEC8xrBJI0XYlvyBX//Vn0zajQYmq+Sb9QxtoipKvG56wNJQBu4GBngkotooedJEZ+QtkqFhD6b0Jx2GXBk7/RKefv5ZrG1uIDUw4iCxbNpk2maFcz7rsYBhm2PhQtWG6chI4o0LpyyYCmK4iJT0XY41d7+WX3YuhVTGhGfcnsf3sdvHfYBIJ3Lxc1TtBZL3c0bu4KISfi2X5eFP5LK47fQNmJmwShBqiBFU6hUZdLgshbtrPhgDBz4fwEqMyWrJrALGVLz5TwRvbOGNI9DvGRaiOfDUcrBc+DMxc23WD/3mB5LN7XVMVSYsC6UkeQqH9h/Bvn17MDU1o52aLVWMJeElran00PK+nabiPe5WOhgE8pP+EINCFc+/chYvv/yyUpO0J60mHTDzsBV6yNu23Rn2OB6Uv1eO2RhyI0+aP4loPyq8J2Y8MJanY+KBfAnpc7LguJMW34f61jXdU9+140b0I0TJF/EDZIj/M+WbR67AxFBJDpbsvfyeDMrFKrKpIfbNVnDztddKEzDC6QtYoa9jzQqIVyszSIoVee6OM3Ac0nhjPooVRXhRorho1q4EKdvhUTYdqePYHBIW2vVg5Xz6H/4k6XaZ5aIt6WN1dVWkAuKvlCLaHbryzIpJUl18xIPOpOTFmlonamRgQJLL4eJmGy+9+KKcLg6e3mGzaYjPSK0ZlVrvsV1kYU+kN7ngI+ryWDWE/C7PiZvN4mJzZB5aOcGBJsfE3VKioSliYcMsjNvzEDZG/0aiMEdIi6SEQxHFUkVZQC4UVaS0U8YBGAqiV8jksmkUc1nMVSq45aaTgobTXpJLZyvoybLPo1IdY+2qqsRLltR1watCtEPdQeYGi9DLtoQ5hTJhgp4jXrcwL/UXf/RLSqdQCsx+GrbLeqSwlLcAACAASURBVGVKEFWFpQB366t5MzpYVD9cSEuRplApl5CvLqJXrOCVl7+K7Z1tT/dZxobCwCR/qGsuWDgY8RASHKFK9PAt8xYPZ7nrFLIeUlAABfprt7CyMoMBQ5mITp1HF5LOz47b43FPPDJc4dD1B8zpm2PFCSSOzs8TFqbJylcqUum5gvVqSWjC+kaUVIHgwHqqsFxI8zrsygGeLGXx7ne8HSxl5D1VvizqtFWrBpUrtJIxTswkBMxqxY6SeOcAmh/i0qy/8dmiPs1dFqR+4xd+ILHuOlbiQlBBXQdy5FSToGDeLKmzQqpUOG/0YpHbvc0EXaFBfhKl/dfiqYc/j3q7hW6LjpgJCz9HDjZBei6MFtE5zrHrAgkL7jYHH4BNCIF2WYQXopsx+LTnlKOUIZ7kxQgeesX1YyG/NpwLTRM73cIWCwNDy1CdcxMYPFxEkiNzp4wkYzufQsD38FqCdj3lmvI0roiVFM52C1tXL+H2G6/DO9/5Ts/W2diJZ/Mlb97JFRKUsZKrCKtIkmDVjsHYHoV4XxjLqRv3PIAcRQS/9cs/rG1n5D9ic27nvPoiiuRMzbgO99KfiANbrR0MhxnsP/12/N3f/SUyDnZQOxiNyJiTzDoZB4w/m80Sb83VdYRtob7DBsm++w4Zt62pUH9qCUVfg8O3/HHs4PAFIqQLJ2/cRxjH2GMMDKG0WxyNE1qo3LLVUTHTx8RPJl9Chg4se9Kwhj2VQb1hiR9OGGu4FF4hjXTSQ7NeR7u2iU5tE//ym78JJ48ftbptItxO+DAGi5mRICMGrs4oRxx4gkwwGFUl6iRDiMpkcxuVNJFdUzLlv37wP2ixVZfsZD05JE67FewmgMOACM5vgP02EH4uwczR2/DYc1/F6tIr9neVsUTLJ7NrDCcaDcKmJDdSEMx+M24OdR12VWqIVZNy4v7/VYzane5lWu2MIUtc7FDX4Wz972x0/C7s9bizpmuz84SXB+k6LlhRCWI8vDzSuRISpRfJiSvK8TThNAezXGE+voE+bWmvo2Cwtn4VrfqWHLef+g8/aowez9eP8geROxBl2KBYsW2UhevLUMlNUbxOyNXyF7wW7z1OqwoMI/WhX/mhJBZUgIX3BIv6qmBXWALe0pPuH5tXyf+dFvLH34L7P/a3SIYNDZxMC8F3TMnxMwJDDPK02m4Lk0wN79rmcFSsPHfXWePYYkxRQWnjME63TJbHcKGmww+I3bp7bbNv8dz83jJ4RpDQriSvzZEv+QxU105CMNvpoU62YOYuV0A6V0QhVxSIwQVniljz0++jTnIGG24NE2ytLmN7ZxXpwRA/+1M/6R0d6MgydUmVbpskiBARchl2bhiZxeduucliCQfWKckjs0aNOCTjN4/Ub/3iv08YQrCaIfhhu2GPYa8RAoUDZ5JvO55aodnroDZ5E557+CHUayvyUoOcR+FhJ0LtdudHEVMW0N8xcgFDMKk6955t4i15Eeo7FkEL57zvWLyAH9NZW0Q5bWMtu8a97XD2wqEZQZtj8Kny7EwFEqgcYdVWshTqn0V0NqHuw5C/njMiZrqQQy5rxREZr4ztscojGQgf315dRr2xjnwqg//4Yz/ila1dLSQXJgoNZJfFErW+K9FKLNp1EBs3pMyRNufnGZpsXj2/mgYGUh/8T9+nKk5WPoSBskm3zJDZM8szx1dzZAylYrhEqtLmxLV49itfRLOxpsExqWDCYzsyYL4g9wVRn5+ntgjnKHZbnoUEASOSOapWGUZb4kv23MEVLTpBBu4cx8/HwZH4Pr4K2Bgj/MeCh6NmKt18F4Ieso8Ou45/TuPwWD6XLig0Yx6/n5D4UGLnS5RLJEZah0JmyQrZNDZXCRevo5jJ4Sd++AcdLbPuipayNAdTIIwDMOGoKUHkfsS4mQptFlrMwBbWirtW5dxxsWUPnPX5tZ5qEP/dr3fyn4Hz2o3suNDpY/KGd+Lxzz+AixdeRNY9VO5wMk0M6SJD1CoUgjhnHja9cgM1DB40ocupoJBCZa42Q6qAT0cPOQb6K+4nNjDWqoPPFQscKjoctPHnDOctBM5UqAmVFbfbDhnVTHmZrqIRvx93eIoOWybHDJChXKRZFyc1hiafvdVGIZfG9toyavUNlHJ5/NSP/ahrNIIO1Epm7zkHyi94nbnh6bYfd5MlZsi4uagNhNx5HkB22pHMqC9P/ebPvz/hgKluwhGKna3p9fAodpOBdmzlZIxKJgJanT5Ofv2343P/9ABeefZRZNJUw6wVtvJdAhGhsg0T52TKuzDKMLsVhN11hEwqyEOvcDYi2c8HkkMXjXr4wKL5WLw5WgDPzH2tGh/f9eO7elfr2K6WgIAolJVARdGinM+BJzBYo6XSHysglLOWNgHJ5stC3bhjudDKQPXbqG2to1nbUi79R37g+1+jrYLepDVx51g5ctcsMUYrLdrtLxsmRqGqGEAUxF1QSprhN37ue9VAx+LBcFJMYsxT3m2foR3mHYXDzhK9ajVauO6d34Gnn3gWzz/xJXQ77NhgHuHkpBXDGxZuVRoR+1kmJ6V8dixQ5K3lhHmMKiKe57HNSfOiAW8UQGecjk/kt83W72a75FX/bwraQ+XLprmDE9/H5JFLxvdxh4emkJD3jDOnZxqShWPv0SKl89o8SOeQVTtN443xvflsVqyXTquOublZfO93faelI51PF4Idv4tx8e/jYwuTE8JhPpDVltNB5L2ClxDzl/qVD/w7lexavbEjVGNNVqN6kQ8RN+CFFhYWwBYQxWIeSSaHzuQJnLu8ise/8KAexpy6IeYXZ71wwOyWhVKmqqimVNM84lPvdn+IQgOOje0raYMCD4/sFheedj0ctkhphoqORY5F3Q0jvZPDGGWY4+JzRQgY6jBaXkdnhQA4ct5zRmgZm+8RIVSM7w1o046sSWPSnzVGSqrLxj/b4udff/11+OEf/EFfbGO2hJNq/lHAqJ5p9HZlaTmHDDONYxa1cdS6mltH56h9ogpUc/BLP/OdymczbolYkzsnVGXknMnbYq8RPvSo1ssTCCwZquX24NIO8MTnP4Mrly+OgILyBInwjEENFQpEzXZL3hrTpq2nWBD+xu1sOGJmUkIhW2Jf2ACT/DExY4iZdp+XvgYuEJM5vtPDHkc0EL5DaAIrKjRGy8jR89BHvVy8dZeySwlZKabOuU4K1cQxy6g0R/dXjqAuuPRd73o3/vk3vHdMjTMnb+2/FPJGaOpOqXnf5mkr7aww2Xh9Rllwe27fjHiC8WypX/zpf5swSJeKYTG351S5uATuc85bjpCF8bEe2u1jmlNNzzFVwvnuNB556LO48NWXkMomyInUDiwszo2AFAvx0t5vu6ydHdpDu9ix8NiNoY7DpBAXd1/JAIxUImGx1N5uY55Q5fE1JinEJa7Pn2PXCuN3vH40qeS5ec45FtxqoS29Glg2+WEquqcL7tGCqWAjTrCXaTTwEVU6ncKHPvQhlUiHmRPbhw7pWBp2V0CtBp73NQ3rFC0nMHCiJdzeL2a0+B45aSwf+In/OyFXiv27SbpXB6IRMS9tOLSyLN7wLpIQUYutBu9ZdIcJznXm8ORXHsa5l55Ft99GOrHWUlNTE1LZFDcurrzMPqE9a0jL3msGtJiHHwAHB8hdoqY3rE5UV0Dz3G3X7qpxg3stsRI7OhY6zAavN55wGXfUYnF31WhMqoFIRtm1/IBSvS41I+dJZLY0uh0nGoYdbvdUkkP1ru5L0XigVMQHP/hBoYCGVnr1ihMTuKjGOHGKkYeD+tmTM0ZiMAatSIteVGkIk7FUhcwpu5hC6o9/9/9J1HzVS2eEgdDekBJM58JPGMhmmOVJI3EUiQsshIv9vAg2II2vrnbxwvPP4qlHviSCvvBqVmeW2LzVPPKYVLOPhhoV8+wRYrxyld96OBOLEwLAWnH+jTtZsbtHBru7w9E9j+3Gw6zxRRy/7tdqgLh3CA0xcj4rd4xahgRI4YsgJ4222Om84deElookje1QFjQaF+/EyWvwH37sx91OBxXZulOpfwrDWmbt1FLL1HIIp1KqhRyGHWeiOOql4zjU9M+aBFohgiGRCls/9td/mBTLRWTUSwQCBZKEKTfr2zGi73oFQ3qw60QpNEmxwRtj3DSu1od48atn8ehDD2B1ZWmUiy6W8ihPGJPFvHEvuAtb64sbPkOYknEHSw/oD0xvM4SGYyTGzOvGZHxtDB3OllKKXgfN7yMBIgFyGz+uBew6VuhOSFRC5zy34I0x2aNIIW190MI+mgOaRTIIO2u5ezstIY1f//VfwczU9AhsspbfFs4JKQvbzHvGbg/AhbaakYznrpW/GrP1u2RM3ziujVMPff5+IX9q0KL2y757vGwm3H2Lei0nPY4hy6HxdFo/yeHxVy7jSw/8Iy6++qKpmEwa+VxWhQfRp4XccF5OdUjFDLpt6xca6pkTHs1aaU85iVTz47tw3KabJTPHJUKRWPiv1RKx2/lc4/cct7OKSZ0gEOxPYeXBb1NDH2eQuhYZjzLsnhmFWeY505QbCklG7Xd/93fjDW94nXPw9FcRMGge4h7RrYmXFzVpnA3rfPQe07DUKS64chIpcKo5G8rsGcnRk1kPP/JgQk/R0pykYxqYMALhnWLbb1uXWz6keeNx8k5KD8JS3VyuhOcuruIrX3wQLz39+AgUoNQyfjS8mXnznpAhkeDTAyR9CxnGqzPi4aJOy0AZE7RQw5EsYYO+r0XG4vOhHcIPCDX7tSp+3L6H4IzfS8wVz+Pzmv2ehakhMCEs0cFR3HkdTZHHgYMH8KZ77sGdd95h+RWRRUwTRe6BZkkOn0cQ0UslFt9Ewtil9PLDWbOMJVG0XWbqeMtt81E8qfT5z9+fsBMv7aHVPRmfigNSAl0XIqmcRXQseLOeXqxgZH5a2DbhTZ2pUcCVtW18+nOfw/NPPKLUpXUpsm75LMfhBLJVRKdjvcJZE8XidoUT8jDNQYtJCE95F3TZ7T8mQqEcOscH8plRV4TAv3fBEXOc+IpESahsmYgxtC3MQGiPuHcsfpiC2P1a9HYfe/fuxfu///2iHhsM5Pdy+rAEMG3PZxTh3TGxr7uIEuwU6Y3reV+WRRlgYk2AeS91qnAiYtC2rJWJbRoCQcIlIivorcVSD372kwmzVjqRJ2vdh1l7FQDEoGt4axSuST2pgsT7blLd+SEtjDFT6QKefOUM7v/E36Fe2xoxIwnAWO/SrOq2u11SZ62WizaXLzEyHXCJiYoJjh0+PtFy1EZJGh65YDZzHIXiIkZIFRBo7HK+N8xULGjYXA1ojIgYAjCeJ45dd8cdd+DffNu3e67AKjZpQ6PG21SpF+2JXGmYugmZVW8QhwgnkjtcvD0nDHLhtHO9k4L5GAyTdxeVi22JKzp0Rhahn0EBoGoX+vfpf/ibJM3QqdPWLstn85icncYLzz6FYcIwjJBnFXv37ZHtaNU3MUgySGVYrZlHZgDkK2wIYwxPqphXlrfw9x/9G6wuLwlDZ5E4ww+q6Xqt7g3r2BfNeoMOKInOlFEI70kRIy8ECXG3VktxtZzH6LliNnZ0ksAYOTGw5JjIWAC+N6jIdoSUYf29riF8/G9CbdpGCQ5f/NAEHCfr2n7mJ39KY2ZhgHqjD/qqTbfEhqVbWYynpvYD48rzFa1GuLBEIlUbzoZ9Y3kBnVDk7SrDbBCNMzqxaYg0mUHhs+ikBeMPcvz0j4zFk0Lqr/78D5Lq9Ax63bYkgdX611x7Eg/d/wkcP3EKi/sO4+WXX0Q+m8aBw0fx8tOP4/ipm3DxygomJyZw6dXnkJ+YQc/JJCwiT+XzuLzVwSMPfUYdE4kzVCtV84QdoCB0yvBASJDiCqtdGn+Zat/9XahNBXoKKSJDZHlmkiNjUUMtj9vmXe+eMazVnekeHpoY08N7sPjC8prjsWqo0sgw/b8/87OYqU6pw7HUvldi8Hk4FoavfFajEVGT2PtCg9gzMS9hVCRRmdzzj0NtKDChUaTxmPpVBMDuzz2rvuUpB+xVquY6lofv+r34GYFVH/nw/0hm5mbVe2t6egoXzp3DnXe/Dl/8p0+qo++RU7dgmcXvVy/h+tN34IXnnsDJ625Coz3EwsIcHn3gozhx+s0oqEVFHfv278fTX7of5cM34S8+/GEsXVpCPp9RO6geC/ac6cLJ4aFkQnpiQcc93rGFJl4VvTsNVCHQE0wWS4wYkGKCQVNjDppXcnqXYOamJQyBKbN6xc/90G7lzus6Bz1Sq9EiOrEMHR1F64OSYHJqGj/3sz+npEh446ERgnI1KgOWX8IerB3tYIJNpkms0Q0PYlPNupMuIoyjsLIxACneuXzBKkM8VCQMbfQuo25Rm/R40kGpKN+l06xbXThbpdCGs/PC3MI8dra3MT+/gLOvfhU3n74Vzz/5KNqNbVx7+xsx7PZx5sUnceTkDUpyFEtVzC4eQnlyAk9+7mOYmN2L/Ueu02IfO3YUjz7wcUzuO4LOsICP/t1HUaMq8dZV9DKFJMkeGUU2asis04QdTmbVIl5HNebIjHunEarJ3ku1pcSQMTVoFY2aPDXX3c1ta4d7VYWS+4RMM1YjxYlnSMjvdz16i5F5P3rXFk7mVaX5rne+Gwf37hsldsLBJFeNY1LbixZPTjCba9i4naQQfk803+NX7sDwJaiGubhsTBC+C7/yOjqZIA1t0si9B6N0e3vHyCNk/uq4Spbx9pD664/8fjIzO6u2FWxNwSTG8ZPX4crFC1i7/CoOXH8bFucW8NzjX0B5eg6TlUnUG01cc/I00rkMnvvypzTA46ffpAXau/8AXnziATRrNRw59UbMLsxic2MLTz76EL789BksXb6sXWGevrMynMkSB4lG191oWZl4q0h+jhQqPgiPfeAujxYUVu/sPcZGoIsd8Cq1SJUfdc1OiJQqde+fAIXh60Md+CoMWiR9o/bypTiYcbP4vEAubQ1riO2Hz3H06FHccMONygqye1TUG/EZFNuzOW+vp13ISwVMSgRRi+LnpfCrteMsqgcMhZj1d1w0CZu34OTOpkIzSDnB7MysasXYnSoO4su62Uj99V/+j4TF6LWdOqqTVaxeXcbhoyewvbmGK2efw+yBa3H0+LV48ckvoj8E9u87iq3aNvYdOI7iRBlfffJzaOxs4/ANd6HEHT87iwuvPouNy69i7vAp7D98rR7wxScfwKByAB/72Mdw+fKyqb2BdTgO+0Xpj7CEoQapwnzIyLZx8Ny1Ukm0/Q5YyJN2gbFsmLXVjOI4LZYxHV6T16ZajyTQbjLFD5rLG7NVbBSP7y0c9DCR2kQcNW8G7zn3cNCII3CcLHZg/7SJsp1lwrCM5nHYbSmKoa9jdKs0+sMu7Y4EgYe55Qs2N9T/1g/V6r7Y+ULOGokjjZqKKNVpiTVfbPbXrKPJDlM6Xbfgba0HSP35n/5uwqpEa59cBM+Xmp1flId86ZXnUJpawPEbbsH5l55Rw/mFPYfEpZqc2YuFxUWce/ExbK1cxsTiMezZd1iLvXzxPNYvP4t0YQLX3vI2dSB89bkvoNnq4vMvLeP5xx8fqR9BmNHPVOwV271c5JKfFMDfaZFzu0kaIWV+Qq86D3i2R4APTxQKh8lLYwngMOHCtKrRjiyhEWaBqcoAddQtSr3COXF2hgfbVZl9NB+DZT8sMOQiqZuTzibxhgEOdFBQeF/ZVPfCC/kSDh44iONH9mNl+SoOHTupnnArK1dRmShhdfmiHK3DR67BytUVnXaYKxZVhdlt1sVJLzAbmStg2GubZnNIt1CqamytTgvVShkNP6lPWolz9Vd/9jtJvkxyoDVutzjVmrGtXDwnZujJG2/F8tIFbK0sY2ZxrwSjOr2gU/GuXjqLnaUzQLGKhYPXYnZ2Adubq1h69REMBykcOf1mdUQ899LjaO9sYjs7j4985K9Q11FN5pUyZOFXWtp9+/Yr3hYzxI8nZlTGn6lo1ZMz2l97VaaFFlSnFk7xWlJvcaY2QaOx46oihqeaFN3XF5+2UPdxhzHUvFKq7jCypo0aYZzUEeDLOFizGzNb7xQV5jmGoNjeyZgEnt56772YmpyS8DY2LmNicg7XnLwJly+fxc76KvYcPIyt1VVkEx4ydxUz+49jbn4R68vn0ajtoFouQIfjFLhBymh3Gug0a+i1TdAIdnE+Un/xJ/8lId+Z+LUC+X5f9pDhQH19BcNUGvsOn1B/tPUrl5EpltUMNpUpYe/ePdhYX8ba2efFtZo7eB0W9hzAsN/Buee/qCMo9p28HYcOn8CVSy9j+/IZJOVF/PnH78eFM+fQ7Rnezfvu3bcfh09ci/m5eeRy1sEvuv30O9bnrMQDYZx2LBXrP3Px5HQZqXrk8Qu8oPCy+I5xrjea5zPy89FFOECX8URKNKoNgYmkCSnBStHGkY9RPDiWw+Z4IlY3xGs3JByhdrLhPF/T4F8ybCmQxw7OYX7vIdz9unuwvrKEKxfPYe+hw6htbKDb3NKc7T16E0rVKVw5/zLQazGzquKLfGUGM/OL2NlclZlg10rejzSpEos1//T3fzkR31nF3XYqnzrRF/LoNJuC6fbsPyJbsaZMFoeWRbZYxsL8HkFzK+eeV0gxufcYFvcfE3l96dXHsbO5ganFAzh6/BbU6ptYeuUZtb185lIT93/606jvbKDR6eOHfuKnUW8P0B9aX/B+t62meYwfCXiwebwWiIiR0CnGqhazdhjX09apM7E1j+VxVRFeqcpFaUMrciAwRE1g6VaDaMPTDR5XcMnioNnIkAmNU7WqMWIDsKHNpcPJ8NLOFfXTdrx8KFp18/ddnnnqfcfl7XtmXGeSqZdMTxSmQwcP4Z7X3Yna5oaAm15vRwvOse+95laZ3NrmEmqbV9H1as7yzF6kszwQponWzgpSgz62eYpvZRKTc3uQ+uPf+/kknS2gQM/RWQ18eC5Kp832WAkmpxcUpNNpo//KTZUrTmDf3gMCA66cfQHDfhPpyjwOHL4OxXwJaxdfwtrVcyhOT+PaU2/ULl8+/6zUYbtyBL/727+NlbU1fNcP/LjKaLa260ilzYwQwKF3WSa/LUlEqqCw8RpimGZJY2L/MaYQ+xh2efRCH722N9cbU8uWGrXr2kIbYNwmsqdG+EaJChiWX62Az1pYRIYvgI02QxgnSQaiJWqSw7KMcdXbTYV90aXJEiZ23rbF/vZ9HMhqHRSkPVRTwTH1UC0V8N6vvw95HajXQnNnW4zUvcdulTlbXzmP+tZVdFtNadvS9B6Z1+3NDaBXw9ryZWvik6RQnV1E6g9/62cSNpnLuo1MeUaF8KBaMOoQlylkeUh3r42GmCZZtdCYmJyRyqfdbuysI5cvYe/hU4JXV69exOblV8XeYAjGU9uvnHse9Z1VzB64Dn/2N5/EiVM3Y3pxn45n1IEvLEFVKGPg/wghEzrURSGbt3M1szxkhXGmgShpgjE89LxnXYLZs7TXZN6YkGRXNdGKad37p9dPDRKN9tSvLE+wYjCCcFlxysW26CCl7gahBfg7zoslM6xsmDvbnD5r6MfFEA7gvcKjC4Oa0PF0AF7DY2p+r2ILfc5r5HrWFLA6kcc3vOPt6LcaGPa7SJcncOyaWzBIp7B+5Ry2rlxgcY5M4fzB61EqTmCYdFDbWMba1SWFqRSwyvQCUn/wwf+YkKhAiaItYvsIhhNsXqf2Dil6x1UZeXYopoqU9BdLKFen5KVurS+hV6/JBMzuP475hUX1DVu/8JIWYM+J27G4cABXzjyPVnML5YlpPLvcRXlmDp2etd8S89QXkhk224l+aqA7TMzMyXazl6p77oasWSUoEyqceDaHS3kbCi4YPVnZzYT/DeumqdFB65HedWKAWlzJy/YjLbwgYChTMlCOOrSAOYK77BtpAbD7RFvevPkJ1pGY17TkhrUXCdqQBMd9iPBfDDJmVScPaAW+5Rvfi/SgZ+ZtagYHDl6PHoZYv3IejbUr6LGWPJNBdeGYmgT3ei1sXL2IAR01xuoTFZSn5pD6g1/70YROGNtIkFrERVZK06sp1JvDKx0M+7W0W5LKYnJ6CplcEd1WDTsbqzqFoDp/AAcOHlEP1NXzz7PfFqb2X4vZvfuxvXYVm8vn1PZyYt9NuLTdwOb6ttAuJUl27LhFmgp77Ta5s7DL6sO5s4lghSMU5bWMyyWILhQcL71QCpESFd6ey0piTCtQGFhTpSMn/WgK4eXMoHmKUhAoETcJgZU80RsPx5Dawzh1LHw0UkR49LxnOHcBgYawBFrGnyk00gxjPVzlHWWzeM+9b0C1lLPqmvwk9h44KlOyevkVNLau2rNkM6jOHQZDO4ZrO5uX0anXrCd8Lo+JyWmk/tsvfH/CKgZCRTlWIFKUrNLLzqygM5GyKkURERkzisGWQ5GdFgoTGPSaaNW20Go0QCeBi02MdvX8CwoBJhaO4NCx42g2a1i9+AobV6By4HpcqvWwvr5lZaaqELWJ4iIrJednafG+ERLxIQmSiEbknCum9Pi5qNfm7jOWqhMTiaDpyGg7tkH88yGUk9fnlIywMLA7sG4S2ZQVshMjUNJDXYzICvW0qHvhhoFbXpq7qOskD2kYp2AFeV+dFb6mTCcSKiGMwaAJX4Ff3/2W12P/4qzWZXrxKKbmFiVcq5dfRae2au23CnlMzh9BuWTtvzdWz4JUETmZ6Swq0zNIfeg/fXcigqHjyAmbzbK7AltLyzYzCc4qA3c2VFCQIJPn+ZhF2XpOXmN7045xqlaxsO+ornHlwsvoNtaQKc7iwPEbJCjrV86i3+mjtHgMm/2iuFRXr1wxRMhPD7BeXl0hZOEpR1ZMRx555YUQLSpELz5Uk9eoBGU9eJ4q11RmxOKWnuTCkCnCyfDzNpyDprM0WJbkvdA73ThegpSfFnLUbqQww05D4PUUQXS6fta3lSSHLQ8nLnZ34O2RJo0jKFyVuYDasVFxxOV77nsD9sxO6muDMwAAIABJREFUSkUX5w5g3+IBLeLm1bOobSxZGXRviPk9R1GZmsH21ibQ21I0pANwGx39PvVbP/sd1AFyoDgwNokXu8MdDJaeplM5JDnLVVN9m9NCmnAJ7A+mZCNVx9YWUrk8Fg8eEzy4fPEVNLeuIElP4NgN7kEunUW31UV25iBa2WnVSa0sL2uRGA9zt6lGKTPEsD806JBN5ssT4IlEskHecC8otOwWQc+a0Kd2ijxj8uDN+7bOidYWK5L+dK7YYpMTpaSHs2aiSWyUNxGv5vENwx6dKPY86arUNpoXtPtdMw/eKIj4dajigIEjPx8xdhAX6DyFoxhCbQ1sR2WaEuy3vek2LXapNIGpfddgbnpBuYzNlbMYtLcUmRQmJjE1sx/FiSo67SZWll5B3rVVNlfEgIWHH/rAdyZiOaQtO5RmGwmiUZ6xIQKsGmVWJqZTVmzOXaiOPEWUJspuuwaob22LZTo9u4Dq3CK21y6jvrksFHnx0CmUKhWsXTmPZn0HufIc2qX9SkRs7WwpyU71yyOQAokKtRyn+ubyhosTdaKNJVOTqUL5QGOlM2Ez6UOojIZwqx+uqkn1BjTMGFEzWJ8XClZeuLLial88xqqETOkEqTmfU5iUVnXnyrxpO4SdziCzXJEAEVbujFad3R1HZYjM4Od8e8M6TmQc16gx+CE0//xdb0KF53snKew7dBIL83sl1Mvnn0ONNps59HQWE7P7VRde21lDNunIBxLUW5kStzD1X372OxOzOVb0zZBLaFTBHDX2CleaMLFQQkcTqNk5Y/Gy7IF1sx+q9zYHWChXMLfvIHrNbaxcflU2ZfHIDZiZWcT2+pL6irAJfXfqGvkKXGweDcFqTsbtUaHoLbSlVjmZhFE5JmLcUc9katGQNf7nwgX9iMQJ29nBJPXKEYV5u6fvMU896HfkeCrP7nGwbDeb1PJ0wFJeKBfrzsLDVt83liA7kKJkhjtYTGTQOYquhMYPYzLeqFfRwcJy7pGPtwaC8iGcEcr+qd/yjW9DliatWMb8PvO4eZrP1sqrqG+tWPuNdA5z+46qgrTZ2EK7tqbjP3QC4YB14hWkfutnvt11hpXQBhtEh6MzvFExALnZWaTzVn8sJiSTD7Tn5K3xZKC8nYqrcy1KE5if36sdtXb5FbFVJvccxszcgjr4s3mMSIvlEwpVOmxDUa/LuYlcbuDVlvWx8ETd/dkf1Q84CcZKwkXgJDsi1uq27TQgr57kLlVhuoTaGTHe2sPOv+buMz67cs6eCrW4Oiv8nCRJOX19rzrReR5RgUJBs8pSMkeiEQl3KtOl7CYch89F01i69jI3znc3X4MttqzDAgWHWmeyMoH3vO1OTFan0RoMcejoKVQmJrFT28L60lfR7zYFnKTSZWlT9UEb9pB0G1hauiRNUixPYDhII/WbP/2vTY37ohqldRdW1NmWKo/M0OCpFFUYsnho1geMks42URaCMITIozI5h8rkJJbOP492s4nKwkHMzC5qR+6sLVviYvpa9NgxMWV8rJ4X64fHysmXSiY1iBAn04I6e9MSGNwd3Fl0jnhdlsFGaSwFNc77oAqLuF2qUud/GeOFcTX/RuFmbRuJAqq58lBqBIl6fM2TiMPmmrnY7aYcp/Ba41w3LXQO++yVZJTrqLSMggdreGMLLSrx6IjqtDTD1FQV/8c736S5nZxbxNTsfoVXPDu7sXEJnXZNglyd2oPK7KLYNIxqCKrwpGSmr3fqdZRLk9zZ36Fi/MjcREDPiVD44+CCtX5iC1s/c1pnhDA+ZjuJtJrCMUHP9BxDNoIwk/ML2GKXgc01ZAtF7D10UiqPP7MNZmX/ddjqG57MhHuj6Uc9DW0RR6GKdiorTzpIuEu7hpUTEVP7KLbS9J7oXLxI6PBZomCdpkjtuHg3jdvqrWk+goIbTQLkoHq7jvGwyey9dX7UGVrcJN4dOUgQ/MoIYLz/anjaUZAoCpXrU+5sgwGN2B9IG1uAc17vufs0juxbtM2RLePwsetFaNje2cTm1XPotWqoN9uYXdiPdHZCm6DXb2NjdUmhqDUw4Jrlkfq1n/y/VJ8ttTFWlmq4MGucrMsfU53y1kX5zWHo3QJ1oEqprF1ON39re0tYNosGipOzysisLZ1DtlDC/P6junnS62Fnex2Ti4exmSygM+Ahbzy1hhMPdFpNLabSrCsrQsbUUbHfwvbahtSikKiehU089ti47XZS4Hi1pdGS/MSByIJleaotbbkVHhi4stulwPhscYCLV0+6lpFH7WQ/2d047H3sFEE7etF4YSE0VmCw26dVrFvaZTpq6pC4W8BHLcCzWk7fcho3nziMTqsmBK5QncUij+FImGhpY3PlPHrNGjvJoDqziInKnO7RaO6g19rRQQHUVKRIsX9b6hd+9F8RNbbzPoTC++GnnguWeo/KSTVbpUfMHizehsIPbGOF8GR1Uk1pq1PTlldOpTAzN4+rF8+jN+xg76HrpHImiadfWcLk7CLWM3tF9WFMScePue0aKTU6M2tTCRFmgsjk5RENje0dqXvBlElw2g1vHq9uDApSLLx2ZZza5+UycVipOh6JyMIODFGf6ScI+yLuxskegqrbgrFbuctD3ZN9kuJCC//uW6/vsb7qTGqIaDFioBikGqzVfDaDt977Nhw5ehS5BNjavKjsI9X9/IETmJyeQ2o4lBrfuHpOY6YWzZd4tGNFgkuKdrOxiWG3Y4fJcjMih9Sbbj2U3H76JuxZnEW5wGMgbGcYsmTHOUnL+JlVVNuSfB4xIftt8CV42MpE2equqxXtNDam3X/oEFaXltDpt7D/AFG0JiqTU9hcX0OhmMdw6jp0kBOjIzhZdNSIVtG2Moxpt5totWroNNtqkcm/G1drt8JDp+xSCBMoHAv4MXaptFLWIFYdqRB9x7UQdppwf2AkiqhBD7ttTiNtOyfDW2RFoTyv56Wz0jKEPcWMTsk5ox7ghomW21UeLyV2ib2OHz2Kd73rnTrakX7H8089La0wOTcrz7+2eRk7W5tqaLD/6CkU6FUnJG3WsL58Fjwsjru2VJkBUkZy5GIPBy0Mve1GVwfDVZC65YYDyc52DZ1uH3vnp7BvYdKci2Qg7teeuTmxKKpVghpMORpRwFgtwqasFbPjuJwoeucKHZIheEYlJW91dQULe/ag3e6iPDktQiL9vurCYaxiHgl3sLJUHaUtZZO7jFlbaDUbqO1s6G+M5UmOCOyZE0Shi1NpFaOn2bynjEabJTNZxc/WoZ+JClOlPG6AgsoiCNavjRIgsJpoU+27rUWCjCDVOxiiFGd48z00H96TLCNUz2JrhWR+AnAqm0elmMVEtYiDC3tx/fU36Pip8ClUxpMCnnj0EQlloVpFv9XC1tplgGeDF4ooLxwWKbRR20aztYN2bUtzRH8qW6yiVK7aCcHtJrrtJhKCQATApE2ySH3vv7o3YTqvR8eDXYa9+ZyqCr0/mb7qRAErLdGBLf2hFnl6ahJ79u7RQSqGaLGSgtUQrGe2Qv04TqJa5Yl5fRQqVSFOxL6LE5PoVo+h1UuBNWeKibsdLQ4dL8boGxtrGrg87xbP/zLcOcJEqWOPkYm4EeUSEZD1awXrrM+QjQfAqgyHKFjBCIUsT2ZhgEgDNGEeOAU3OxbZ4E1r0MvPTfL0PyJnLhhWnsPr28HqFMZKtYo98wuyvRN54hCb6LR64gIUJmZxww03jLo+EKmjKfvyF76AieokSpOTWuy15fNqbstoZ/bQtfrabtaxvrGiEJbRMdkz1akF7XpD69qq8GFYxnFIjdP3+vkf+iZtEjZmV6rNCXW0wZwk4b7qprRbtald5z1MlaPyqg4V+fnpPTOzM7j2uuvEqCAIYIOwDj4E7SNVqQashTkkU0f1WcbqFBR+JQOD8XOzuY1+u6OfyaYUB9pP9RXgIgDD2leJBOAn7vCe6YxVTPa7BF94CkBJlaOBgKnvJ59HqVbadfNfmC3Ty7NbnFUlJzy2Vh8G92tYp8Wdye4Kx48dU/NZ1p2RYXLoyDVoNxs498LjSPptEGsvTC6iNDGtkwXjUHoWPfL5udiV6pTCrPWVZdRWz9uclWew9+Bx45HvbIrlQ4iaY2r3eiiXp1Am7yCblT3vd5mOrqtdds6Zralf+YlvVehFhUz4Ubli5oVVAdGjhTJnw20UmV4CKFxN8fd2Gp1liSIG5c6k/TLbbwT9bsfO/5pfXJQ22L9/vzx3kh6Ge06LVkumZiQSqKLIrWq0ttDheZs847vZsF2tQ8GNzMAXcXsKJl+BSRND77Pdh0jypFsVBcwwNOFY5ZiNjk00Z288V82Ja+zU7JgI1rn5ATlk41II+PXUtdfhmmuuwebWGmZn5zAxUcX66jIaNfLF+rjx1rtECrx85ln0W3XNyfz+48gVyzh06JA0DL3xKGp89OGH1fF4Ye9BXL54Dq3NS1aDXZzGgaMnNY9rq8syZdnUAM1GU2dwZrLkBvoZpMOekk6N+rZiciat5KP815//ziSqIuwQUivoppo2NTeCeXczSqPOu+pY7b834ELagQkJP/vLSkkNmaOU8e+0pXSoKCjqMcJMenU/7nnft6Pf2UGjZWgWsd3hsCe8emdjw8kTLQmWtWvmrjWP02yxOZb8T4I+zzmhGTFP2QiJKrLzDglBPxpRguh3iOPmJ+QxqZKy9GppghqqjLfde69ds83zQbMoVytaTFasVqozow5Q3HV0Lq+/5Q70Wh1x6evbV6U5D5+4VZNPPjmdVDsdyMptv/DQQ5jU4Xd7sbWxgtrVc6i1apicP6bUMcda49mpTXaeaongQLw+V54VtVspzWSI7Y2r5tekmYqeMELGf/9F9kET3OMkPe/d4VxsoWVaLMNwhdCovYNpOU2hkhCEuaPO2tpRmJPDybfLqwGxeox6aa4awQzVpyWXTuPU130LtjpsoleX3SNEyd5xW5tb2FhdQTLoOH5uxEIuaqdDLNwiAnnebPQeDVr7xLG9/4rCoYHIlJEGDWhW2pr0q4nyqE6d5ufmm2/GwX3k0PdF0ZXjxRMH+fBeU85Qi1jC6soVHSBPUn5UuzS3N3HkhtO4dPY8Bt06NtcuCTy68dZ7sF3bxpEjR3RSImFTWhCO60uf/zymZuYwNbuIrY1VbC29it6wh5m9J7Bn7wHVfK1dPS+NOzs3g1aTMHMH+cqsauTps2ysr6K5sy56mBrv8Yhp+kh/8ts/4H3QbCFUye8Hh9mC+lGAYyfDKhRLeeMcnbgzVP438F1CjwJivGVlnE1l8pSo97ZMgxPuGPqo9CYzgeqJN2qhGVq0CBgM+qpDI6mOtCjmzDfW1zA7M6NDaKKihF2XVP/k7TEMJCGyV1S8ywklXYgPTRvLF0/lLZQKKGSyuPGGG/Du9/4LhXWdTl0EfkPlGBV0lQ3kiwwcqnU+Kz1fmbp0GitLlzC7Z49OGZC6L2Rx9cJFXHPtdVheXkKqR422g6Tfwb6jp2RCWFBRLtuYTY0n+MKDn8P0zCIq07No19ewdO6ryoQdPH6bPPJOc0sHwHaHwPTstNLK/V4TufIMZmfmNa619avi3ak8macPq8Chi9SHf+dHRottIZf3J1HHwziT2k5mGLEhBe0ZnCreGp0kPyhUjEo/RMXAA5oDU+8Ww6Z1noaYrN7OcgSqDFNo5efQyS+g2W6g120pxqYd7zQaaDV3pKZ6ZL2y1kq4vbVfZm7aTtyzXR4ghQANP6ScEOTMzDTWV1clnG99y73Yu3efaYheG7fd9WbVk3OxL1+8LEHrdpog/6xcrSppEW1G5Cc455sTWd/awMziohaRqrY6VcXls2ex//BhrKxela/BoorlC6+iunAIczPzYHRSqfD4KFPj1C5c7AOHjomHT01QX19Gq0Ou+M2YmZ7FkjgCqyhVyRGfx/bGhnh9E9N7MDU5q8UmgsYTkzkHC3v3iU7FRj+pD3/oRxPtwniZiR21QTYQwc/zEp4ah5fa7uBLB6V6laPgVe+sFDndKGS3YwYtAxSokmBFaQ1ChoYuDZmTTU1iY7OJrfqmKE47m+tsrYB2py6An+8jt9zgyzTyaibIrhAFUW/Z8oKeN5242s46zp05o5OD5YB5XzPrMgS0egNcunwF/+67vwf33PMmdfl/5pmnMTc9qaggSn051kbdNAjPqpYvkIJUJ/GAyWpVOALHUSpTnW5gbnYaV5eXsdNo4Prrr7fvazu4/ba7jSY9wR7ljAKsCPHBBx/EqVM3YG1tXdy+2uaqophD192qg1fPnXkG2QSY2seESB61zW3UN1cxtecgZqbnVQ1y9fIl60RZLBnbKE50+JPf/qEkCgREY/VWjdEPk7syXsJ5/Sxt6/tlQqKe2+y0pNaNFAw/US96aXpvci66drtfUI4Z0SQ/F5rHJUl4vM3ygWtuxeKho3j2madw4eISVq5exZXlS3Lc1Bd1dhYnr70OxWwa1UpJMXJc3zh4ea8qoZcgN13OA3ciNYQa1w/TaPUH+PgnPoFbbrkD//7934/6zjr+/u8/gce+8iVzbPw4BjmTxKjzBfHv6E2fOHlCLBoVEKiYzzooMKTiTQnt8kU0jZWdWyR4qClRWTa7Up2wolB30D73uc/h5MnrsHR5SVU4w14T/e4A+07cjG69jo218/IbZvYfFBeP8DFbWk/M7cXePQews7OB2tam5fRlwzkHnpn72z/8aanxAOwjTKKaVk9MERVYrWidjvRSQsEWNGykcrFjjdnMsTPnbVxpWBtn7zzgxxf1ujxxqCTkSCfg+HX3n7wVB/YfRKu2jVy5irnFPejq8BlDuRhFMDR76cmnlOyQifAyXFtb4/AG6udDdxKenxDkDNLBMAfCive9412oba7ghWeexSuvvjRKDgk1pBZKLEMXzeLJsKEfEXRg3mNyakr2mKElNYyYs/W6wkzGv9RGrVYPr3vDG9SEiLmJhKnWYYJHHn3UBHYwRLtZUyODZquDI8euxfLlC+g2a3JoF/fvw8b6ppVZnz+Lyfm9mJmdx9raFW2GcnXaDnuX752oKDD18T/9Oc96xaLEQRu2IHTVY+G4+GKMyMZ46exoMQ0UiMW1isZd+dC1YrZdnYcNZ77ZeG86ZXOUATp43e2YmZlDu76NVg+45uRJk3T2YvF66VaziacfeUSTZbVc5L7HgY8mbAGt8jMqDBiZJdvsSln2SKIs4u4336MzPK5cvIiVlSVD8lhPXSAtyzo5jkwQixG8S6OlVXkd4tI0N9ZhgYJAweDPtPkkVcq5K07ge97/flxz5JhCKAI/HOcjX3kEO7UaSjyLs93E1GRF9fB0tLrNBiaKOVXDTs/PY3V1HYcPH8aV82dQnl4Qf2Dl6iWU8gVx0phfiDPAei0u9of/s+9sSyJwN5jjZd0LvARaDlks+rhaJy4rmk5sei/U293NVNbet2t0wIqfejvWEE622lmgUTZz9NQd4kqz9HRzcxu33nan6EN9LwgkiEsy4PNPPAHjjscZnS6oLm3xe9M+u2duywt2fjzbhPLnm+5+HTavXMH66gq2ttcFCAlhcx5ZtJuyyfImc+54RuPa2OWMAthjbhxyVeTC1hq9Pk6dvg33ft3XabcGBflXf/VXsb25hTvvuh0zs9PSIoRl2W2KHZwD++dYGT9rnaghU8DUzDQ2NjbF0WPju+iwVC6woH8LqU/+5S9rZ4fKDRUbReheyTc6fZ04ehh9U6XehMa98dHnojmNfm9N9ETrkZ0mxkwN63XVbvt1cLiK3kzLnLjpbhRLRXD38nD1O+96I5JhV8QH+ges/OA1n+VikxDo6dlx8zFuRsxRsVMLOOlW62VsWXK3KLQ33nU31i9dxubGGhrNbSUQQiEpDeu9xSJEDWaqJYeM/x5HJGqR3dkN4CoqRukLTc0v4r63fb2gz26jJkH8h099SpwAopTtVlPPvr29uUtXJmihA+ZSgqzvu+8+1Ld3UCiXlG2k+aht76hogI6q2Dre/Sn16b/6oGlXV8dsnRFVhoq7YWCFuFGOhu2abtsZHCQJDeEcGcgSoIqlEE2VxiEzpt9JXrTT4Omhs5uQdxvy9OO1N98tpIxNbzc2d3DrbXcDSR+dtpEWCMgQwHjpxedEpzWYNHaupSo5vjixwMa/Cxrp++iE3DcTdPr1r8fy+fOqH6cTx6DTHDM7mUDM20gWceGdzCAz5R0gomOSiIuuScRC8ffaGEijmcBb3v4eVXU0t9Z03ccefxy1Rt2Yq85eVX23OkuRjGnnoZHvTu4AfQGdlUrT0TUYuNu2UwtOnDgpp3Bxcd5qyD71l7+h0Mt2HA8xsSZpRKFMPXtxwKhPib1P6tDroQlUkJkSXXCDdWEPz2YzfmqdN3qLUMwOHkvbGWx8qQGvgTH8/ckb7/TzNbjYNdxy613I8HRf2h9fbGLNr778guwcXxEh0GdQBYvzxU2VjqnwMSxAdeCevrrlDW/A0pkzKmC0fqm77bkoKrTB6tbsr3EUTjZ9LFctyFjQoh3hZEJj41AkkCvjbe94L7r1DWytXpEwPPfC83aWp1pVG8AVTXEZbYRGMg1h1SnBqOUCc/HJ3AmyhX5uNc0p/cSf/1qiRQ1P2rsKEQZUJkdlMFbgZ573bvM3O/PKbqgDUehgSQ17LjgcNnfOwlFidkgagR2FoxhdYZA5TKQv8+up03eKSUpEbWNzE7fe8Tqp0XZzZ+R4MYw69+orst100kYayk/dNQKGTdiIheI2llpD75fmsTHfcMeduHzuDJo7NU0QkS2xXvzc6+C0x7OEBov7aq60820xdGBtHGrLa7Cu24PP3jCNe97xbgyaTWxcPa/fsuecAVCR0DGuqti23lvNSpssK2lA0mudYwaaIm26r0HsXJnLB//+vxso6lAmOwT7Jhsttv4uAiJ3+lj7Z1eJRtAzMMVjldFiCK/2npzhrTOjxsEqc+axLwWHfULMKzfu+nU33+HYb1uY8Onb7lSIxpZdro+lwi6cPydIlU6aqVNbHMX10VB+jEQYioQecoSOAfjceNedWDpzFvWdHfMxvADBivt3SUu249wshB13tW6pYkvnkshh2IVrQ/YRVTjIurIEb/7692ix15bPSdjOnLHjLWNnhjDp7G3vrhRahfehWuecGF/d2EVc7DA7ETnIdHzm47+XMDgfSv34PyfmaZF0UhzPf/RmMxa4CfHSronuAj6ZvImdOGelqqPJVAdfO+A1doEWX9CrxMkaqovsZ6f63va6N2Nnh2yMLlbX1rD/4GEcPHgE7caO4mpRfns9XL50CVubm+Kgx3LwOgQ4RlI/5liJTOiHoclPdDVObXP9LTdj+dJlMWnIXo0+M+HHBIEhTvIbuWxxGq6r6NGCeZM+Cz0t2WSwM88USeMt73gPeu021pfOCjc4f+6MLbZ7/+FjKKtHAfFW3LbBDGJVqYo2kB9O5+FmNCaK45hTn/rb31EMUSyzH7j5nYb5+jmY0TpSYZLtCd5InQ7Ey7JSHCMKGL2YixkQbOw07QS/VrAzQ3p1Yg6rJxw2NcnN4vSdr8fm5roQI+5sxuF33/1GtOm5wjQQr7G8dEU7W2fZOu891DMfSrsjcHkXKIVSLqD8W4BJR05cg621DaytXFFPEiFRHFsY9TFnVnVZrloDHYxdZ6cGBbRsjeN3Y347S6SHDO5953vEe1+7fEaLfe7Mq4rVJf5+T/lI1ppAOL11d6TZMc0YZA3RrLxvfKzVa6KRz/7D7wsuDXqNUYqNVmyOWCBj9tCjzkTqG8qdGylOs7k6scZzmrb7DR5VViv8Al8AMUIlheYV6+jBqCbVzn4TVtdW1FNlbXUV3d4Q97zlbei22KbROvJz0VZXVnHl8mVRbCOc0iLpQBpXoe4oUXeF+jaBsNEJ8k2l0Wy38cd/9Ee4++7bsY+JDR8bif969miU4/6KnWoQjFwzcdG3xZJAMbN+JFMQHYnLI4Ove8f7MOh2sXLpqxLKC+fOGiHSVf04UBU5i5G/4AUOfA+F3tg2u5z34BGYtkwj9bl//OPXhF6jvp8uwRZnGjFg1NGXUpqN8yzNSVMxgSNmYZ/ouQZyZuc8ewStE+fNhpla2z1wLVpPJEkGt73uDeKNE3VaW1tDu9XHvfe9HT0S6nqsDrHFXt/YwJWLl1R/TafFMl9GJjTeuFdwqurFgJAwLyNAiAxTb8BnThaBlK44dYahu332tG8cZ2k70M/T8uOVAjnUCX0yJxae2nvjUBrqoQze+Pb3Ydjt4erFl2VzL104PypTskNndzsvhUmKbBvVeFCYAwCIsNds9Wtp0akHPv3HCZvEcbEikRF2wj5odjeAjlGHP8XGpto5SOFkyrCYBiDqFUcbSfKVMTMzoZN6vM5bu+s1xQnWYJZlwjfedieuXFkSAZF9vtge+g1vfosQNMba8fCbW1u4dO78qLOhjd+gzXhZZskmWlThcC69gI4cPOLyjCgsRy0RN36dkn3m8UYyJeLqEOZY9N1FlTfgHrlpDyvCsMZ4pC7TQXvj13Nn97B66ava0ctXlrxvmrFr4npxX9G8YiMyeRKaw9GeCNMsNIOyfqbKE6Q+88n/mZi63T2OgWzQkPgIAeiI6Wxt503HJNruND0tD9CPNLJF9ERJADY6dshaPlscGWrcvGe1+VANOFROdN0Nt+DKlcsiGjJe5K3uuvtNKp9ts10jGZnDIXY2t7C0tKTF3t0NnJTdHSV17tWRHKfxvmynh1Dy93TqZA+9twq/l9fL8NLHGyf0CGuIvqD+jCYg9j9UXYAsdhSym0hWtaQzeP1b3y2zd/XCS3LKrl694nQwW2gzpbsHxIiE4EWAHOO42tZ9RjlFrzVztFBj/cw//BFnWotkDEmLcUOiaHPU6DVtao7F+uqsMmYDxxeetczRRYg2kLHsru0O6lOoNNMXcRC7YlI/gJ1O2613vh6XLp5XcbmOccxkcdfdb7Z+afXaCPAgAHLxwsXRafajSXK0xjQNPK7AAAAgAElEQVSvh0puasxb9zg7doUgVMMR5Pw4SCP8OfBvPytr5MCS+KB22t5wncczSSgClTQCR+z8kXBwsQG84b73Soiunrf4+tKli6MTl0zQrKCB9xcnnKiemxRGH6G2Y6FDsEJj8hoSCP578B8/nNhxjP7gzh6hNx8XEgDiKpHzF2dHMakfGoEDVmd890AD4YrEF+fT4j+2prSzSEjmkzepigqj5cSk5PMl3HT6Nly8eAbNWl0IGXfg9TfdgcpkVa24wtPk37mzFYo4C3bX8x1pcn0TDiHVdnw+nMj4uxweXyA70NVACk+YasxU9zIjDIc8XtdZ2wolY0fSNHT8aAr7tKAdJX2ETeL1971P110+94IW++LF82aHw79RGOzZRvWIsYPkLTHz2ub7Sj2PHEKzmnHagFDSz//TR/ycdPPiVJ3IAckxsA5CmhTufH719GE81CiTNLbIeix3vJi14e6WpvAMWZgIo0BZmYyFDLsxOG32DTedxoWLBDi27RhmAi8Ts7jpphuxvbkyMjU8Punc2bPujVvYGBy0sFcGUY6Lnjkv2oVj7SflTwgxtL9FoY5Br6aZI4YOkmOobd4rMoYyYd7VP7xyhXBuhzWSYYJjN9yJ+YUFLJ99XkJx6dIFT8zsEkkS1xaMDKKq1Ha9JX9Cc4+bFX3v8xtRTurBf/qI5mA8WcBBy5UXROdsEpEIqZbd4Pvp8qPdYS6It0o2BIfgCr/GGV0kPASiEzF2TJCpmzghwHb88eMnFFY98MBnMD8zrf7m7V4a3/QvvxU7G1clkRScdqOJJ554VIsklE/OmSNebqujowHllTnvXZ/EBCBsXxAwKBzWsM6OUQqKFT+vfi2+ix3NlyCrSCKQNkcIzY8wGrOcRO+faioshfmD1+DosWuwfJYdKmpYY6gpLWKJFUszO1FEWDjPzbYiC/V1k7Aa0STmdmS7vcFQYA2pLz34vxJzauyhTUpt0qRu2GBdyQlzZlQ3xPeN8dQIpqhk1h0fE9rd3t4SHnVGcI/WVVnYwlDdcX/aTd6/1ezgwsWLytpkSK0Z9lBvDfHP3vcvtLPpuHCR2IjvySfI8DAVqSOYvSWnhMpNk7xgn6jY/fKmvdWlhWzWuzvUfbBrHdUd/T52EcMqdV3gSSd8U2g+PxMkujSquTZbcuq4rOixDmTKU7iLIea5M1psljqNvH47RNPGz8+Lym3FDPaKGF5++2ixw2FmOXAwSCTsX37of8lmW7Yodl4U5zP+cFBE9un/a+vanuuurvM+siXLsrk4zTMdGAghJc0Y22BjoLSZ5rl56kuf+tfkodP/oy+ZydBppkmAkkkoNrbBKdB2aOMB27JsS7Isy/iiy+l8t73XUdEM2JaOfpe9117Xb31LXYzxtLvTwR4pSR9LgEZeVpvIk5QJtIYnSxJVoAiPCgRAGTpVePBnQizc79H2pJ1+/e32zb11xtpsf3n8qF358ss+WSdIVpLteGFyvWrBs9Gx1QzLEJWYoCejJ1QnF0gDa19LpQHqjKhFJoxQa288TyHYI0pGTcI0abtzi+3Ea6+3m1f+pz14uNlu375pG68hOVhPcdqonJo1wXvt0kGTyQ1zlMRifHEtAgP/+MN3kgrhZuGHkB580V4nVu2D1nSxWD8qy8zI1O53tZh/opU2C0nPO2AFfxbJfKjG/Sc8JkA8prHvc+2Vk2dZDHn0OM342+3alSs97MgIKJ7ylAvLCU6uoJuqMgVQalnjmkZYpU2W5jGO3oyI1GY9RamedAnPKBgBlgQAYrQBrquDMNd2JofaqTNvtLWrVwiWYHrYqNVoGBZhzHmukM5OngfohMUh19f+qCAUT57ZynO/+wWRKnFociFCiJ3qRFYLtyAQwOq8k7LtG8fESlBX4QYt2u6nt5kSywXWwpBxCKrTIAeeOEnQjG1VgmeunX7zr1gQQC8TrgPM981ry4ImdfuVCYBKZgw5hC0WsIGLY3oLLbBKrqlmqZ/NiFW/p+RTAh5SWaP6ugaqmwpsu/7tqlfSpTxYmKh+qJ149S0WQkDTvbGx3hEv40gNkASzcp6AoEepYazVuvMe3XYnawc1HrTJCFdU4406pdfZbbRjYdNAUkpt63Pao0T4kvbMueIGFqpBXYstG2SmJicpFFZgrPAAMOq99FyvvfmXpKcAVQe5UnYet6t/RNVoh/9WGFeRMlrsLB7Xx+YJz8AowA9dVTun7iH37Rx6pgNFjQOmS7gV/BHWA3TiVD8Y3j7u1zeIc7vAMgVth3U92E6++jaZHzfvrfNkax9k4uJYZk1xVX6vqGrlPGBf5LDFXPR7JtV7/sN/0TmK+q07ZueAC+1eLv1dthsnAMNJ1K9tUJ5TlXJsaj6nPJ3Zi4C9Vi+YHERsR8hnnLB3rK/TFOfxe6Cu/s53ScRD4va97bb89dV27x7w5KMql7q2RiaBv7Q8g/8aAVdoOODFiU6kqFyT90LSJynwJPoeJUfOjeiD2uwxO2Wp0Y3yReDRo8x55s2ftDsr19rdzVX2d3HsYuaTs4xc0rV9/Sv2L1UwPKfEQLG6BtoEmzf5+KNfWhvY1ibD5FOZE231L3XI/8+Rfjqgh8R0OhlyukAGD3uM6TScqxVbvSdmhJKnV8HERQeGPSyJJvGhaBfCxbz1wlI7eeo1MiHTmWq7beXqdQLzMk1eWkm7O4odKXJhBomotjnAVKatV+jkUIVpSAyPFMbAjqzNkkJNbE2CeY+TyGQAMjoZuqy5W/DEVeAgwufAQjvz5l+3zdvLbXVtpd0Bu7OdUzw7ng8jq6kNSvGoh4LVfyrIWWpVb3YO8uTiuV8RSox4MN7zrPxLavIL6c5E7hoLMsKA2d9KzMffcy4XQkfaSrSpGqCYe8bOzXrII3VL5KYF6e79x+3tH/+EuC1K8nSPNB5Qgdg2fTYmQCpdXrQ96V6lEkVHHDloCWgBYMz43LGHnPGl9ClOTNS3snWKh5FnZ77dzh7Sy2Ql3tPAG8wCwbVFSARPQA4UNvPlk2fb1vptjuVYX7vFe0k51CaMsgeZQNBDMK19F+p9Cgx97TzhF8//2o19Q8fFfZcS1qnqm20Ok3SI7BcQCcDYJHrDO2itfaiGOzaGuz2ocJbgaSAAsy+pxj1+z2kSXH9j61F78y9+3DZuL8s32ttt6+vrbR1jLayZ9LzJHThvwFh40Fv2iCK8KHZ8sAEsBvnm2EBQhuTa+X719mkryc6gUcbpfcv6wCuI40n8gEGIWOOXT73RtlZvtdXby+3uxpr6203Bid8H71miADwLINQcBxFHLQ0Y2WQntKANuHbOo0w+Pvcr48a1oYq2ZSP6ifZb4nvzC0JW5gTq1CTcGDavxsg4DVBlcsaCWvUm2rusmiD935BUeLOS2O5Cte2duXbi1TNtA6dgD1TVjQD61bVbXaYZYbg2YQnqJ7UKKN5JVJcgBhCsadaxlKgpdBTIQYKZcq4SStKOEh/6AbbjIBzQ9TAZQAT5aYHSlaft+6+cbvfvrLW1G1fbPYApe11cCS4Wh+y0Yj16+jNxvN86BzJ/ZjGgzum/fPrJ+/TGe87XKiRqNb8QFYV226ouqtrdpz1mBCI2T+p1oCFHBDAECCafaUerUiRzmFjh3E7QcB1qr5w63TbXV0lnhc1GVeyOwxY9B3qzTBvhWLg/X46odsZwXyWElFoc5EGs1ZcCDXVdSrbOlxPznjCOZV4lQsgOYZydfADhzxi5USUJRPjD195o32zcabevf9XubK5zs3ELMkfVAbR+NojIE08cJeKOJU+/x7etP01BiAAvXvgNN5ujkKIyi0cH0Bq+hG5UjRpf8H2wAbFR+3PN/Ey3s2Mel2J6PVbCL17fTkw2qsezOiszNeLJ3lw7ceYNOmRomwEVFurda+urM2FXMnYUqHjLAe7vW5nkxvPtekq0L9Ze7DEDoTxoLsBtLt61aB8mobxW1G5GfDLxEu44ok1R25cX/4MfneD1bl77st0hnQgcOCFMD3pONvYmpLYH5kWwHy2SZ0a/WOJ/ijsPixIstNkXzv96mrSe0p0eG8GN1WXYQOAZzIEWIc/dL+i71RM/CgujlDjgsb6uM3bJPwe5mQpVct2Kaw2AJHFKa6+cPkuqRoyMPAjH78GDtrJyvTtMqqPbZsXw+zlzOpMAyp8Jl7KIPZal0+I0qHMC1BzklgFJkNPNwIQDaMdcuzppoImY2vSJls4ZAEccoOdefJk+wvWv/ov1akQ2nLyEWjbsL4afu0NEiS3BrWhanOaWMI5iiEJJ5eO7N/7Jxfd6R8jMD913NfqmZgvwcLoYI6ePiDnzCnbDyRWqcn96tGqB5Md1kmvHpU5zCHPTXMeOyvmF9uLLJ4hU2drc4MlGFm7l5o2OF0tdW0I3SADY2xVOb6NjcjK6SQkg0smLaAVqtzQxWoDU8eFChVU5N3TG+ZTDJg2pJoqOI2tz7cixYxza9tX//ne7ufw1JxbSbNmHSpIIDpmG2TSSDsATUIg6Uqj0j+LQGrZMDBCe8dNL70+hluSAqBdbR9Y+kRMgWNioA0gKOwVdyYEdQsNfWlajgns4ZUjTQFoWtegFzKbIRimRoahN4Q2+xEwoTTO/+FT7/kvfaxvra+yUQBsQ+LWHRrFtdMIoaVTxgkeQMJoYU4+GY1nbd6qmx6IKqKiig/B64z26AHf1OTQaPoj2KHGrylZn+Pt0Z9ouf/FF+5uf/rTduHalXfz9b9t3jj3J+QfJjDG9y5aoxmgGIEgWeTxsjvjBRDhss7b/Yx9BDt+0Tf5w+QPS1ygLlLgl+12a9N0JghoqnAJwimUze2xpG8GUnoefiUZaeCxtYkIi60Z6uqlj25O1vOm6Dv8ywdaFvftb2+21s2fb2q3raqnZ2WnLN67xwYW8CdiwJhZ1/yAyldQaoEQKMdWkCzelb6tv/AgKVE0y5EfCaEfSCy7BVP9XNXFxqOqTra7ebh988G/t5PGX2xLYEiDkOLEGIdAEGlARcGgQrorHkdUDH5oig9Tgtd6mOMPJ5oPkQlalLKCzJQeDxlE8iJ2NLRinI7ZbiyeV5nRy/xMbqhYVLXYqO/SwS3IAzxLkClUZF1D57uScITo725N2/NSr7fbNa4T34HpQ4xAOaJioZIQq1AxpKS7v5yBToQz5VTCkVJuTtJqyqCqQpA5dHUuxUth/KSldLHFKwqoejnC2JksYpcB32d0207JnDXAtlQxi+AZ1jfEW2zucQwZoFt6LnSPBCYDwxxXL6lDOL5joCKFXjZmT1sTi4SEB36WtsXTizxj8bEZ+P6FSTz06hNCNh6qUDRd0SDEkXtQUlS6Q8HeceZMwZdYXBEA/Ovn6W+3m8lVgSLlRt26taHE8CObbMoI5BTFVaEmqz68WWzk2KnP63YkBB4/aYqfPBOYMX0ySlNJjDVsxIE8lysIeGJw8b6TcNZJO0n6D37xGBLTNHALPxXArspklQDO2s0NOuHtb95iKZqOCexnhXzFE+8OnH/Bk9w2HNDlbJVumJvpsthIk+jyrRQnF0ozmPHPQL0mpjkoQZosM1TnrIOhfeDC8PPovgi6hSvToIjiNsIEnz7xF/jEAnHEfqPEsdGL5qPP4EdFYET5ojapOa7go10WFGt6fm6PWpkQuNDJOzECFIudO79ydKGSz8xcFLSFpcQiUANq24zjajqMxs+manKCnjXCR/RkEufb6EYKCkpSQMnKrqYjDeWXZbJbnAhEuD8JeLmdw6oZn07PxgiHLaWHzuGdcRp0GKEBuEoP60BbcwwID6HU9WbugJ9FZwhAE6plqEz+bbz9CL9gaxkI+pucKB024OYdp6QFmbV5NinjAePhpeNMzJKmihnvNDpFGUZSQaESCykDHTfrcLJxId7pogfU93Pewiz5xDHNAcmDI6eJ5nMPZt0BZ02WdsjXSXhJysTS5X85FFDhyqk62Ptpicuniu+JUsXwn5qZnTika5bO8XCQuajwbSu1g+yhbaT0SRKUXVQkUdW0yBjX0iPAbniAFD5wGCRI3jIYKRNdcIWgP+sGfnyAPORiI8LV8Q0R1GuCq6hKEjjPLYJON6aID4znaCZ34bwq7bDcWcjbRkky6kiEJtxiuWhBjfxlaudFR3Z9qicY6UXNgpMbhxe608eCkJ67jzmd5YeL8cfMOmDQXc1p69+hen9pbBQN/R6jKwfCXPv5N3qKoKpXWuHnGnOUEx7mQsyUvOw5RVB3SfLAb8sQ1mTYmS6xC4u5OD1QnZvP1gv4Erhz8pVWNcnQkVOP0QHvm+Re4qWBTwtfNWyukn6A3ySxWAAvyVtP7VHFawZlhpHIydTpxo5iT5E5MQ9VG4CvXe48qm0yiT5WRPemw7KwUtuOBQDEK4LFOAqn4OEVtx9xWf6mPniZ0GcIoAYxGpq2HULDEabWU2LFWpTicmV8KnZhata2m09BbXUZlDJ/FaKI0ApL7k4wOJTwxL3naUxcwjQf5ZJ9u3BEErBpBLCRIQiqGRm2+PfEn323PPvccqSTxhRInrscMAMD729tkG8LG0dPmu3gRDaiP/dVwtREbd3SttRP+LSEbBQ8+OzabuYKR/lVUEpNh6k5DruCvJFNY07Cxw0Go5ARjU+P9x//JhufgAcwoBy5Jd534oZm0T5MLH/0rq1483oVdIBs/c+xl2fqm8WYHNMwktQWcZHCNcpSEpYs5Yo5zkMqW4GhhUapDe5EqOQbtO5QJCyEhSsjWOXTDS2AMIRrjTp89S55OfA+c33BQOILJbI1KWcqRxL2hbSKgSiIp0zcSOXIKs8AAEEbFwjT1EK33sMthGrWV8W69JOq05nAexeeuTXOiaF9KF9eMNoWwc/18GPJs+TlOblXz6XaJj9A10acX3p0KYTEQFUmu0AmxPY8nrGFPQwTojZY4mZOBZtKecnIY6/qUZL7IiKPtnTvMgfCgiiU7rWIB1ZDVssp9ILcDWO9UW13RlN6Nu6tkEEJ2j+zDYPhzxSxISy2iMk4anrrN7s2kN9PrhQWiEBotk/KmzMFgYooDV52umLeo/ZiebDYrab16WMD9xdPucbK/V0NevAM2P/kJYO/w/ELhylzVCCsagDabF+bpHl2JSONFv4v1aFRRdDId4xkpCjyV0psD6Ie/0zFQykhT64o9g4MWPDeegW4ZhrK5vpzSphZ+FDUEPFTv2Cuvnmkr167y5e5uronczYkdqjE3K8ZZVNyMcBJOHGrSek+ke/GFgkpMC+7BU4TnOuAikWktYeOl9r35hjhp2BycOxs/x+3MetnJ1MFBfludKTBP7Et3eKf9MG0XES0DRcRN5vQDHM5RtIr2JC22U8JB4cSBnpz78JeKswtTLz3yvZEZktrTw0hy8AAOLQy3ibSl8Wx42cp88TTCMwTkx4uEFRmqBpkSXR+4NQmF79VhROJbSYQA7rXjp063G1e/5qJt3d8gYgVCxdKsNUV6oiPhym0btEBEKhZdqBipSxHQJ2rgOAr3VGX+p5Aoo3Ajpw68brovpBFrgPdmehmzxgszFKpcMS34LBNYKSfjul1/SqBSWuY77Gl2N67fSXNc3NFUxZiWcXhpsy9+/B6LnWH94xksqqOnMp33jqOGFB4+BqaeWdugGVgKbVBnvt+WOO9aJzfM/iwPTveYhMClU8+G972I4kSHEkNbiJlQEjq0x/bOtJ0+c7bdurHMzQH98vr6Gm12TwyRqQnZJRHEQjUne8dqUkh7Jgca5lknjGKumc6oHDe0KjOGR1vSA00TTn93PO+0HkOYMVtLGyikqPyA0e0Slatr6oTCvMmpVVwvhKlgVPiKiYRgwy/Suks4a7TUEy5WL9xoCEnd7NjQ/FCGXW4lZAWSGbUGT5eDUuz49MDeN8DpTBtwVEzKopmDOUhwR4GCqp+w370+sD2AgIAIEepx8+cW2osv/Vm7uyZ2QHCRX7++zDHInNG5s026aPGaisRWeX45atgcYsvIqCBHM0PQsanyDVwx8nShhGVDaOVgIfqginU+H825+uwBhoP4PLBkAQlkrSEQ2fCUhKN2c/BynWQy8X1om5rBjOfdVbYrez22Z+jFk63TkpvGkajA9rSuYlIffh7JlIqEIKiYEs8RN+8xcWcDVp4Ym4CXxwMDyYm5GrhGkitwsLiAbmLTiXHNuKMolZR55pnnid7cxcjG7Yft9q1bYmBIWLgLFWlqjU5eo9HJQXsQLmQikRAJcBNcIOEkQA+HBSgCwgh4b4bajd5ybW6yWlgLCCiETHkJYMWlIdI8iaQLGvmjqnFtrgNO9UzBTodOZkbTCuTfKIGEZ4BpwM+zrvHQuwBks2OL8+ewJw6H7IFCF3Ni3WGoZn2JamR4h5HIJF6wcHHgEo7lMwT68T/E0wovSKVpcLwkVlkraJP8nDXi6bQdXnq6PX3saRK9ovEdDhoHssGjNEpDmkWxKE6HpuSJ7opwXla0RPADqUtrUJxJOnT22IMQSVO9FlKsSAk3Ewfn5NHj3xZB3UxBCNqyF5ZS6gUEWQPl2CJtxAvuo9hfMXRYDpPLx/tRU1mYoE0gBKHepM934fy7PY5KPJYTJifdRZJCCSkPO2KnP6v6CF1HBCcaItAibeDwvOvvihpT6UyoRhVCNB4i92WSBO2rjx+3g4eOtGf/9Fm2Au3ubLfVdbQEyfFDEoV14eku2RHiiCoxInADrquKuatXCBMJbHQPd6g4IVydiK5kt6zm5YXvtsXDmlVK/8CtuVgH2VRdm3l+1w5U+VPuQRnFsZZsP8JweAsl1gyjkbG+bFAwVGvUuZXNSddJNDQTM0hqZbOTcYlKr3ajH+GGmRaa5BrpRYkwdk1ORkhsArcdUJ44cvlcEgVJFQZUgJ9jQznv2qMaBpOCFTrGP8LxObjQXnjuhba6uiLmgqt/5IJT4OLFp5l9H/BwRssYANE99vCrOvkD3nD9TJtBzWGzpbDQwm+kT0LKqNfkGhA2xbGSI6vWXmUItykETASlrm6wJwWyx+HGFITN2Y2QMHS91h60ivMkPGBffPbvU0gWbqzyn9R0Xjqbig2A5xwg/0gc2GlzrjdqpSaEEuPGS8y196dgByugVGPgSLGjSSRQLbtmjVLn8eMnCDaEqn3n5//UfvjS8/LaCb5YEG2XB7+HmUGU13a+vE9Y8NFtOcq+FE6nP4n/DkOzt5hajuXLAtLs3RwqCPW0rFOyma3dq2k6QqpVu7ukE81mMJo1BIkPWKNSviH7ldw6NWlICwsMmg5aJDXNbPhw3H1me6aN9ihtMREAOQAmijfAQGHUKEAkNSoEptCQ+BPCFQdCp1d4ctko3XMmGgj0Ju01ZleEnf/nd95pZ86cbv/4Dz9rf/93f9sWD8+3xUOLnB8GbxueNuNSsCog/jVlCEMbb3TQKR0IWPq7uA1u8Y0GDL02n7Hi0p0jTZMFO1fpvLoNyZzobAVWQbiXJ5N3p6oHHYjbh2nWDJcCQzPeGeu4uLRkLZsSrBy43vi/73RPLl14b1pZimJ/ZZMVf2MjOLBlH8mNPlP6hVPJ8bG+u3G3PfX0U7LplHrFhUlyKMQTLzgkP6paDs8YDRmTEuHA1VSSVC/1Y87sRBPhw3ZwihLnNz7JiIkftKUlTNgB7xlCL/V7YeKuSAKM9nSbrwo26ekOl5uydez88OmjlvJ7xjbG58m/eZ0219bW1zgkhtqFhRiphK6u4/OUHEc1p3aKmJRK0Yoh3aNHjCggvNG0iumFQuUhKpypk0sX3p9ubm4yoTCcrlrBksUeIL0JHSV41wn6ZcNjmwPzGaBD2ShVYSCRrF512g6hNdNWo8+FL3WEY0m8xF/garFeiGQDxiIjiy3BTCZqfjIhXgsoEKxv4lRQXfPkmesFz/fNN1vMpYcbpfssLKjITmcqQA6CwBpKM6eDJQjcVEa6s1vmqGSjKRRutpDGEeZOTJFpNRoeU54pthtTgZL8GTBuJ19szyM0vBc2OxL57U6ZbiZ77hFNpeEbkqVwJCeieucSfgLj+u8rohWFpuJu5ZI9ycBCoSyXwQ8u0EcYR5Sga89hlBHnj+gLagxOk3LvimnxBRN3//5WO3xoUaB7xPHz8+3QPOLgbaVQd7XoOAAYldSnHIw17/6M1kOFHsKDwEQcjHotItG+ptgj4j/AhHDqMMeD/kkn1TPmb6YWoG5PxuNYN8dPoAUPlmCsDZ5JPDShCoFJo4N2+ZPf9s3GpmdTojKrg5bNrp57PNrYOth2Zc6GdqAtBidocN8Zv5S5GS44xGEj1bJDF9zTfaSdB1Q+geJ7OVomk7U9xKhGxZdqm03SvWYI8bzppWIee6IRj/MW3m67HSaBxTDpzhyO8RwqicYBlUPmvHRYD0ImaEh2h3V11gph/ygwKI6Y3A4nPp8VocCgueRmylPrzA7adIV9cFjjNPJk/8fl302JPCzzr5SEGHTGRajlWboPORs9q/5lnxlzLqonKaceJy1pPZ40Oyg1BOLfozatQUgQU8hsc7+Mn8pmRwPd37rfjhw9qkEpHuGgbNkA62Xj6Yi6GY+x+67CIWwe1b5LuECSJgYGGPLOnY127Nix/2f6IgjQz2n4i9qWdhnVO4aedvwQdiE7FzPFOFzODu8xYGI2qRMBMzmG8cA8w9T8Lip5iXhkFg4wvp98eumDGXxCbHNOeAXwRwhy2hmse2J8atjZCHnYvU6mGZmeZ8Eih73zOEP99+yJ8h7FAcLCQ+UlYpAfIMHqwuZ5liNe1/35Lv4c1X3meblJT8+g08HMFNbYyBPlx3MPwZ8hCIFSJSunRFBoJvX5/VqxC2k89jIlKbZ1HAZBmxSDay112jXgHZ+7t7nJwg5VPFuD9sQV68YFnHx8v5c6ocbjIWsBRzEdL5qXIpDPbSfDSYqNnG2pqfYDf8c1qhbQQBi03oxMnDzYQTyjQHH4CBRyjDGiFtImI5SS1BvAaK4xLBJ6v2BSxvuMal7i+TwTFjNdILDdMDlhJkz7boQ6WMpJKI8AAAdhSURBVHeFTPM9/Rqn7SGm2TLZokWOZ87nJ3wJFTxtWl2TCMY4SHD8nO9wf7g6QhVbU70/gokKBbj8VZk1NxaWfAk1xOXLv5/SPhtaEw6x2G+l8gZTQiQvdrtWYvAgyYpF3UeAcpry0hEYwXoH9kzJj9mxilGfta0X8SbOrainFL5xRkhaVL0IQbf0Re8/l6DqkMlOjAVPn5g1aY+5NQmIGss4M5qJEPO5g0MaT8UTrB9ULNYFEUzleckzVXufE571iTnVeqpfLHYYzI442VwXLazv6VYuv2tMwOSzzz7iZsvDEyYq3mtuPLJiY6pMNjvqvnrrWqJxklIQiGpXCJbWnrGxuSayXimPytFTokYxcwowOfXwgBH/Aq9u4rze751JQGFuHAmfoDxiampdOUmdYQORFxdiFT8TJaZBfGFWNudKjbBy7RD+5tBwhBRNgRJSWQtBqPT90cwY7nIsqPP5ps0A4RBKuHpOTQfsozhKQ2OHlGGz8eHqqWbzUz8epzykqFC5QY1kY7Upo+gxWoaG/R/9xFGvtQ5bncR45ji5meKjk5ci/igYxPGSWgRXqVOdTswM4cvfIoiBGAffpsORcIr3Mxl+/02364hFQdGLBFuqM4DGrBlMFd5V5rACE3WvmkmMd5/3UM1cdfZ68GifbVblAMuRC0NEogL+jgs+9Ds+//xc51SpH0p5MKiObE6kKDndqp5rPbyq8bHE+lskOLadoUahg8qmj2sPxCfGIIhZUClQePxaCBPjwvbbYQmNNq6TGrJSkE7d+lQmWRLnbzhW0tUiBxi5+pz4qn6x2XHWlMMPBNgJmd4TDm4ZIV5qwTo2/969LQpGZ2xy/h73TBkzZgIags7XnCpd1T/oG02NZ8QrNjtSk1NWN50pOvdJMzXKAWUhtk0hAY1pGBAumqmqKbJww2kbZdMqEJHq2PiYAZkQJVeGV6xTgRQu0SX2/BGC4GVUsx5hTH+GjGvEe6BZgfPHFCb2cMvJnzwP/qQ69vgFePO5djZoqOtBWJDTCUEJiie16W9zziJAua+c2j2GeEAE6T2Vas7BgBMatNDsgTKYz45sYvfJF1+cFw9anddRSlYjoaHm+AhGbJaVeMc/V6ejhh9V6rT4aQ0a6jhCNpw6lDrdb+wifjYuzxsBVSZPSQdWoAwqYJxpZ4mkcalU5cSYKuvBw4fUEuRutIOVEI4LzchE+Paoea/GjI8Th2q/TzLUveJkkcQP9RxBzmZn8/P9CBQg1keOLLloFKbkUaHTvjjTZh5Xric88//8XDZbLrw+GDWkgsUgcmNhxMWOvExV9yqciAqK0GSX2YT+UP6bed2OIEHixm1GrhvHo8c1hkerNtZasKnhHTZDi2xwIBGv0DI6BQinDh9eGsCA7n8Hj65wCM+IpEo2O2iQnETew5oDahYLOBoAM21wIGarxqwaLhmxmouoMbjWAKp+ND5mPaJpIgSgBHvyyaOMtSHJ/YAZCxw7zh1WnA0vT433mT2ZBIqw0XoBVprc+hNtkOZb/Vt56H5Dj3msKoZ22JmsEepI3qr5iGceCR8/F2xoVqWbu6yGHkUooRJRi0fOLoBJBR8WPlflWBErPK54huQa8g7yA8yYmNGI1hJxxMhs6CRLTqScqoH/jg+E90h0UgWY4bCLRtV5zufzp1S6+VFNeAAPPbTfSSbxmZFBq55xJEc4LcGH5GVrI0EAQ8fEpzbSmbId1zDcV2bQtVfWwQL5d+gngCiJk7V/w7UnmQ44xk50zeLwUvH0MDNYhEMkiEOodJA0mouHl8hJokze6GGTf+DZIrPGr2cBq9kQkFBCzejezmWEPJue39H1k6cfEYUEwKEVhxBopHUEJEIg1a4GSp1wMSly0KyjBX7fh4BTfQEgdXMh9hICMJMujWRp4VVPjuufF+nqPjXYzgIgz5WntcTY+G74TmP0qTWcqWMt24akdk7GpkvCR9twTnwWJPY/mw2nJeqf82bNTMgcOMuhYBnU6GcszsEF0UzVzc6192ukaBeZORMRWJtFSCMEw2fQy+XfEhTXsn0N2nN7/DtZF/8shy+Ck/tqr9CSrGIINS8STNCsPjwo+vJQhEwAanxspLzrYMJif+Nc4PuCz6rmTKkMrpr5ZJUsuTlWCTOJd6vW1H5xX5QZM1YqKjtOVcITLeAgxgkvSxy54cmbiNbsDTwnlPgQ9nlSoPlX8axy2NCgGF6xkf2iBpvF8/YTHRUPXtCcQDx3nLrYeTbulRFMSHAwDGQXrUqwOKXEoO3stKWjRzsQQSHfWMH8HUxK7D1zFm/A39y9KenyaGlV3Kmlocbria6OQiS7OkuxPbKD8F71QJ1+0r9E25yGP6u8uvFU/24zDYlrdVjiE6g47+S+a+PDdAxgdU5U7CliWXB2Yqgc4LoLwHujros6d6V4dmGB7feO1SNssPOY5Y2vsXnjpPJeU+H3EhYpATL4YhB/R4j7oeImSVvBK4eNX1wQ5psACg+hjQboPlCiJm72nAbYl0oe7TS+7/73fRjI9n85OQ8T7wFtAwAAAABJRU5ErkJggg==">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -832,7 +895,13 @@
     <xdr:ext cx="304800" cy="304800"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="21" name="AutoShape 14" descr="data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAHsAAACkCAYAAAC3r1GFAAAgAElEQVR4Xmy9B5Sl2VUe+t0c6t7KVZ3TdPfM9ISePIqDRhqhZAn8DMu8hXnPmGXAawHCZDDmwUMYk0GABcY2wQSBSBaSQBKDNJpRGk3OQTOdu7q6ctXN8X/r+/bet+7o+fbqVene/z//Ofvs8O1v75P6ylfuTwaDATKZHDKZDIbDIdLpNHK5HJIkQSqVQqFQ0Fe++Du+n7/j116vh1KppM91u11kUmn0ul1ks1lUqlV0Ox19bjAcYjgcAAkwTPi9XYfXKxaLun7cm+/n/XuDvq7fbbfR6/X1Pl4jneZYEiCd1ec5Xv7ni9eIMfIavC7vw1fcg99zrNlMBvVaDYP+ABOVCjqdDiYnJ7G+vo7+cICpqSmUy2Vdj/95bSRpNJoN/Y3XHQx6+prLZFGv11CpVHQvpNN6P+eB9+X99Cz+lXPG8fErr93v9/X+mAP+rt1u6/7xe36en4n38JHHfx4MbL1qtZq+JgO7ZjabQbFYQurRRz+TJACyvtgcDC/A/5zAmKj4ykXW4g046fZ3CklMLNcAyVDvyWSymkDekO/JZCgIPc46uFx68H6fP6JSqaLZbCCTztjkcuFgg09RQAYDDJNE10mlbHIyubx+jjHwPrwff8eJiYnm2PL5/GjSY3K5yFxwjovCx89SkPj+drercU9MTIwm2+YgrbEUikXdo9Np6bq9Dt8/0PizuSz6w+FIiDlPMU6TBKDVauna/Bs/z+cZF8zYWHr+VErvp4A1Gg1sbW3pd5VK2TadhDBBqWRj5TU5tkzKNif/a30eeeSzCW9EqaBUhzRmMiaNsWt5gZAwDoSf4QXGX3wgTjDfpwE2GppkLn08kIQ+AbLSHKYN4sFarbYmm/fkq8MBZzJoN1vo8/tsVg+RzmYwMzOja8YYOAl8qPHdHRPJa8Ru5vslKJkMEkp9xrQDBW44sPFo0pEaCXOz0USn28G+ffuktXRPLnCvp89QSMoTpp14T16f8xC7lb/jz3x/aAj+HEKgsQ+GWshWp439+/ePtGyMnfcZ9Hsab284sE3A3ZskyOZMI+dzuxsxFlnP0uuaUHGxbQdkkMvGg6eQplhwx2ezI9XDwYeKp3qhpPPv8Qq1rxtQLfUHSHH3+04P6YWEwXYIP8Ndwr/x//b2ttTOxEQF2byZEk5Es9mUFOt+aVPNMRG8X71eH/0cE8txUfXHK8yGFjpJkKdK5GK128hkM0hzTLwfhaBQ1L34GalvQIuhuTIjos/SJHXaHZTKBY2fgspdSIEYN4tUrRT8MIn8Wwidmb8U2u0OUukU8oXCyByFidI4+n3kc3kMYLs1TClNCe/ZbpugmrkbjjZNMZ8zIX7mmYcT7hqqU74K+bzZwIxJTbw4UP6ev6OEUgVJsoecexOOUCGyYbk8qKz5no3NdQ2CExFmQjug29X1ymWqnwES3xm0vnpwV/cxCqp1jqPX7vBxkc3nJQSctGq1OhrruI2L3c3J54Rwgig81CBSdy5wOZoPJBgkplI5YVxYCdtwiKYvYJg3PsfOzo7uqUV0/6DdbWsecrmChIjCzvmlLdd8pmyhzBylpJK5cfjM3ADtTlv+QzzDxsbGSHiq5Qn9jf7EuGngfIdW4XxwLkJ1x9+kbb/ylQeSMp0E38X8pe1YU9vhjPHBeSHZJ19sk54JORJUg8WiSbfZNu6+oSai26V6tuuFitNuGZrTw50sByudNtua0KY1sb21je2dHZSKRRw6dAirG+taBNpH2ihKeKjDuG44llxYTmjsjBi33i/NQ7tb0PWnJie1O+kzFMsVrK+tI1/IY35+fuRvxFyMa69mo4Ecn6/T0Rj17IlNfKfTs53X72sjcY6pwQqFnNQ+BWVlZUXjp/ks5vJaAy4kf8c55e/54nzKbGbMNNCMhXaKv8VGDBPKcfLznA9qPdnsxx57KOGH292+VEkpbxKdSnEf8UY2aDpwox3mNjkmOLzyojsLcsiovodDPSQH1u31sLW5qZv2B2aLudgUECrJGKQW39XpoD+UWjOv1zx/Si2FiLuF+jSdzqDb77k3PpQnigGwuGcR9Tq95kk5W/Ja+wOZjjTv7d5uJksHic5kHu1WC8ikJQx93y0lqdTE7pGixkvrs7LJYcYonM0mVldXUCwUtfuSlO14037uZfNGqZTsLn0AzpG0B4Bex7QOhY8CxMXms/Kz1CKT1arMDl+r6+t6Xr4nbDMFM3yEiFBC8MOZTj355BcTqhpkslJFGdDB4ETa0vZ6HQ2aaom2iu/lhHJgfJBQY1IX3M30SD2Ei5Aq7DE93xAgqTEP7ai+5Xi5d08JplXs9xP5EXxY7cApk9R+zx2gQR/JMNEC8R5JYiGWpCexHVEsFTHw8IxmI5fNabHtfnwiap8ChoNEO3B9Y10LMj83p5+7rbZMVofOkdtwOUU+rjATw56ZQfkrFNi8LUy300V/0Nd9ad/Hwz9+Nmx4q1GX2s8Vzcni83CMVPGcf96v1WhKC4bDG+8L7ztsdcyjaVWLKjS2Z198IqFNkgT1uihkcpK8YWKhQKgLTjofIn7mLih76KAwhwvsNl5T6HFpSLWkjB6jS608U9nOtNSSpLvXe02IRBulsML/ZuaFXrTZPE6IHoKeJr33rsX0nFhei3aWO4LPxWeKUIy7k2q81W5pJ4a3TO3DBdGOTZuqDDVqiwp0JVR2fwvV0nouhYa01VzU4RCFcmm0q/nMNCvhryhUpUD7HAlTGPakbrm4IQAjjZBOj6KWcDLNL8iNsIoILWOueL/Qlvydnv2p5x4RqFIulc1uwzzbcqkgCTdny8IVOSeuiqhCQqJ4oXBcQm3JexwMMOngQ3jo3FUCWuiM0V9JpxRiUUVxYSOc4PWnJyfNi4Q5TXpQJCjkC/LaeX8+JD1pxrdcKKp4TmIsFEO8drulxZVJoK2mk0YB6nYNtODOd+eQO1iefio9MkXUAAp5ej20uh19nhM5HkoVsjkJlRwlmqGUCW84TvGZiGBoMrtde26Fn7Is5vxyTOHAUaD47KGyuXBzc3OvCWUjnAuVH+qb742/6XpPP/eogkw5LcMBCrk8mrU6si6hqbQF5IWCxb5STZykUsnCKk4Mna9koAGN7ARBAvfeIzzjoLk4dPT4PqpIDmK7XhvFvfzM7MwMWu32KKzLc6L7nDhDybiLqRppTkpFQ6K0A4e07ebwaVe4g8j7Npst/Z0mioJRqVb0lYLNC3KHc2KlGt1eT9BLdmSO9+ecMIwUltDrax6klRJaDQN6KMC8Hk0HJYoCxleYNOogaaFOR5+nNy6zZ2/D/PzsSKOG4JvDa6/xWJ6fD78gMA5uAqGh6YzubethplWLzZ2hsCABOq02qpWKSSehR/q83ClpAwG4GNyx3DGx66QmcqZqAjyhMNTq9dd486PY1uFBugU0B4VSUXZ0HC0at4+h8kIoQ7VucXfT4XEAQ0JZNGiXoZs8dtdMXCyzm4kBNPTUM1TBpgWIehEmrUwY3KmFpOYo5PUzr5dn3I+UaRIHXei48aXQldfu9qShKFjTMzOjiGZkN31M1BS8PwEbLUqhgEa9gYmKhad8hWoObcnn5FgVkfR6Ei5uHL4/5t6wCEMWBU7Rdxmak5h66tnHkoBAOVmUODpOmXQKDC3MVqX1gFT18pZztDe2k/h3gg0UgMCF+X6qND68QhXChfLOzRSYM2UOoL6nL0CwJLHYnrY2Yn/6CozZOdGESTWRdK40Jj68LZjtPBfIlMW2HCvtOHetoNax8E82t0sVaVJvCF0GRPEYslBI+FwMnbhr+ZwUBMW57plzgTkHfF5BpA558rliXqYqVY2NWobCymcNDcdn1Wd890tTMqZniOvQzfT0tASJG5DzEoJuzrAJGsdvttxQtRBwrolpV4tkUi+8/IwjaLsgCgdEEF0OBBfL1Qe9VvNg9QtHwMzrJfTJRaEKlQfoi0nEZ2NzwxElG8y41MbgLTGRlwoM3Jzf2QLaAyREy2lfAallhm2cVH7WJm4gf0A+RD6vhSKerJ3q3jd3KLUBF1DXSlnSRzsjbQ6p7bAKehJYe1ZeK9RqxNpyHtMGJnEX8sXvhTJms2hw0YQZ0GegYAwVj4dQclEnpyYtOeTTyvFwiiLMpRAqWnL7G5uEfku9sTNyOu3vKdn78MCZhyBIQ8xEavyZF59OtIiZFPIZokwNvbndaqBcKGEw6KPoWLW8c0mK2Sg+kOBFd3CUpZmYGDkFFBpqCmZcwqYp5u6YrZH5cODGMjp5CY2841xOmoVj4TWofQK14wSGdqA24WfDWYoIIkIcU30ptDud0b1kagbEx7N6BoEghCzTad2Ln+H9+BniCwZYDLBTq7lQM2IxRDGik1TWsk0Ubl6bfoZ2snvcMZ4AP8zh7KM6NWXJIvoXBT4/zUxfmkJ+1MCwBjqTvP7U9PTImTREzoQtwmD+bmS6uhQUcxilgV4++5KEiCBARmrUEBxmcxT0p2jPbUcRXOC2swU39IuCwt9x0gjtlcplhWHh2PDGdQL8zaYGPlGZ0OcD2aIzxJ/lpPCaA3P0qpOTI7+B15eEc9CDvsKi8GojpjR1Y1omJpYIFe0bNUCn05ZfEF5xqG6ZBU9cUBtQi0i1e+aI9k8qME3YNJGGKJWKSIa2kLy/wKVCVosRjlK/w4wefYMsCDYF3Mz3M2oggra1tY2Oe/Czs7MygxGXB6bPZxF27iqeP0sQ220JFneurunp1LDdYSIVy1PLyWY//1TCC+RyWYM23bGhyrTQimogh/Qw0c7iwwp6c4mykMrsnh6eNtRVeG1nR6B+2DA+CCVND5LQqelJYmWvlRk1eJYf53hGgMWQKnoXiTJNZHlzLmAAGgrhaNv1ecPCeT8JL737HLFuy3QxxuZX/p2LaGAPowWOlwtroVOnZ37G0L3xiCzCpvO5OW+0n51O10wLkbY0Q7WugKq+A1S6n4dk/IZhF6OOgKQjvOQut8RMSiqcY+dzxqbgnEYoK83nDhqvR/vOr1wzCgId5Ugppx596pEk0Cthub2+FpXOkGDPrCUMUkyMM1HiMabCINlXUyN0lCSBvnDcoRQMOkemWgwjpvetzJDwdMavGUkdFzqIArHLLRwkNErEzAAOLgr/zpBJpoC73L3rVqcjIeHc8p7joQntI69BoRHSlBhAxPHH/ahOI1mTTpl2IronGzow7TaO7UcsbOrUEibUVFqklAMy/S7o4kWem8/ATcB5irCJX/lZjpfzwu8j8rFM3FDzzh0aYaG0WJ+hZl/+CZ+DIhs+Q2g5aVHOMX2OrzzxsBabEs3kAzOblvUpyIYw7JG7z90c6kJwqKl0hWeesjTPkHivQYMCMnyyeE3loxXSEK60XTk+6GBtmP9HreK5Y4kZUKvtaLG1kxxk4b1MJXeVaJAQuoaIxRMY4lkrM0kWr3Lx5StwEvs9MK6mA0cVST/DQk8TLu2uMUcp1HVMrrJ2SSJvXlEKIxJh8gyxnGDhmTV+Vo6TmxXZW0LGLoiBuMnhYx6AGEOwcTx219iYMWQmMaITwsaDwUhg+RwCv3zTpB5+/MsiL5hX20POSQv5vDkuXGzFa2RtkHLjoRQnmw+hz7ojQlvHvSc141SkwMM5cE4Y6UWUQEocU5sUsJBCxdF8KAdPtOMUqlhYRc1gnrQtgMXLWak8MyW0nwNPF+6SLwK8oE2kAIQTQ01C28nPa/cS5iyUNEFcAD53eODhcYd9DHAj7DavG3FxhEImtDaO8C3CxDUaNWmY0A5M1hAj4M90TCm4XGgKJ0OucAYDIg0oVQAPYWeaNUfslDhyUItaMfyY1GNPP+pMFYt9mSDnhxrNuhaYzgWlqpwv6uE5iAjutbPH+Gjc7bSLyiyNATDSAo6XCzcfZc2C/ODok1N0LMzi5Nv1OB6OY2enprw3BaxQKJoal49AEoGBJYwciGLxPZxkqr+AGyNRMA7YRMxLdWjYQErXpSaIxYisGxcu8PtwgGKxKbTB6qGm0AJ4WBhUKQoRx8+IhQIsP4SIH59xLEbnNRk2hRMs6Nk1JXludHjDBNIp5Pt4T3EISH4grE2giBh8Pi9TKij3iWceSyg5TGVyMFnu7I57fz2qtJYgSdocTly+UEK5zLQl1bqF/nzI0A6GsBm5kDtcUF/CHWuYeAAInHCCFoa42a6MGNESFvQwzQwo/CAE6ULEh+N/20H8m/JAcro0CQRcGC83GqOxxU4Nr5XPKgH0JBCvx8WlL6A42Yl9kXjg89GX4c+2aJaIiMWmg8YF4hgopAzBNzc3R7loOYtyuIxXJ6zdSYYUNGooJm20OMp7M09uiKRsuzuIyk0QtMmksbOzbSEI4+uJsogYEcJFXB+OM7GD1Jce/aJsNrHtGj88HEjd5tMJup22EvrJYIB8sYRSqYzSxASq1UmUJ6Y8xKKDYyqf6pA340LRVlG1cuI6XebELbnP0IYTJKTO0Z7AfkfeKBGxXneESAkJC9za0TeaAJoMjr3bY5zqSBi/IoASU9nKjrmpUa7aKVAUXu7+yJ5xYiIk5ELyvzYA05m9rjhoy8vLyGWY5m3ImYpEBdOvBw7st3yBzBnnxeJ2vm9udlZ+TrNFUqUJI22tOZ4MpxjimQOby+cUVnEHVzwCoqqTQJaK0mB8z6WLF0zbFkpm5sjedSda8+Kw68hmf/mxLyX8ZaO+g067jmGvIyZIPmcTORx0iOojRQaGXPoicoUiKlML8gRJdqA0kiJEOHUwNFQqGCfaCV1yy7bk/Fy4cAGLiwvYs2ePecEOH9KeinjgryAdctdzh8euNrtkSX9OEAkKVOMUDl6P/zlew9oTQY8kSWSFtqVQKhSxtramu3CMAUhEJDCeOQo1zK9rq1c02advuwOf/Ohf49a73iCHs9M2XDoyf+F/MKdgmT9T54pcHCfgV+IOnLdxti43bbtlISIXmxrXHEFuImozmxyxiJIEa2uGIzBvwfmi3S+VLWFFTaJMpUgWBqumHvzS5xLyoNu1bQx6bXQb22g2ami36yCLI5fLmFpk4l057RQq1UkgW/IwKytUh7TeoiQsh3K5guGgj1azhYcffhhveet9MgecUE4+NYFiWIVK3EGkPNmDmUNkHjOFicTDRsPIhJxsqubAyvk3OljdbkdmCJ6WLOSpRSioxptmOElSgBZ0OJR65cQyAgmTwPtywng92UDPpIWD1WvXsLm5gTe+5W34o9/7EN7zDd+MhESO7Z0RHsAJDQHu9Q13N66bRR1yNDNmvgwhsx1Oc2eQr+EMNJvUKPSsFW45Pp9JG75BU8DfUROb+bHsXIZhpwSKiaqszKbRr90UfvTjf5Vk0n3UNtfQbzfQbTN+LYgmw1evb+nMtHO4h4yrBZ4QB88jTbJDvojiRAXF4gRKpYoGJL5VviDItdHpeVrTmBOBo9PmcMEIhHCSRdFxZC5if+4+Tg7NQLvbcWpSRfE3QyXa2Ga9qc9ZmJdCtcpkRV8U2vg9J4PcdArG1tamcHZOEjNh/EwQB8JciF3rW4mfbTS2UdvewA03344/+59/gG/51n+jzygJJC/egB7aawpKs1l/zZgsvcp8g6U9RcaUo2lzIoFwX4S7lbtaCaLQViOMwVk5bhKEySeGFWTyTEUXTJspbBsI8qVzq4TLX/zZf0u2tlfRqW9idqqCen1Hu6TXG2gnKF/NZEQkDpwJkmT5YMwDTyBfKiNXKCObLSCdLSKTy6BanRKVaXpyGps7dUPcFN7Q4zfHy0APc3I4mIhZd4n+fVQqEyIMcFE2tjZx9uxZLC0tKQ/Mscnm0oZlcyjm8zh27BiOHz+O6ekZdFpG/Y3EA2Nnzjb9kJ3ajpH0U4aARXjEcZjGsR3HCadz1GzsYGdzDdfdeCv++i/+DN/2r79LGiLoxeMevj1P1xiwYv0MtYvDJ1EWjQkPX/TAsoMsEk5faDja+OAO0P5qw4CgEfPvpEQXjXiS92oRYhTOy6P/QPuukPnDf/rBBANOWBubqysoTzhJYWjlJ5Q8euIcSHjc4chIEDI5qZpMtoBMlra7gHxxQna9Wp3GxOQCElJkCcP6i+GdqjGodpBCd2ATzAdReU82JwDlxZdewksvvYS1jTX9vecxcuzWcOzGVfHoHtz5JUYPBczPzOL06dO44/Y7BOoEZYcLFHbbgKTirsOWSrQjDB2DdnV9Yw2HT1yPhz57P97xvm82E0LOuUyMOUfhW9Cho8Mlm8xQivj5iPtmi8fn5e/DmVVenqZnQAEzDrrSlA6bCqyhqePadNoCkoQRgMCNcpNmNpywqSSVo2rSJb/xKz+eFLLMTfeRY/oysbonVmGYnbGgPC5CO0Q3n1IXjpI8cd0ASOdyUunZXBmV6iwW9h7FEAa+iKtFe0ywwGNvARwYKmy5cPkSnnnmGZw5c0YL0uoZm4NaRQ/ioVKABLHYoeqCIBDhEgkVfHCKFBedCRSmGMnEvOmmm6QFIg7ns0Y+X0BFwsXxWjKyaTZWsbp0Ea+756347D9+Cm++712iRtEfMNNjfLjIm9PTjjy9tJrnlhU1EATSHBAM4WLtEhW5Uw1MIQ/Acp00WSJe+m4NoCSfI9RMoqcnnpwzyKRPVI44XGj3+LX//P0JbVKxVECKnGXmdJkA8cUhmCV97xmeqMXiLjCuuZH7hCwxFOoPMTk5jUw6j/LUDKbnDmFyZlG5XQoMUbrI1jIuZCjz4osv4oXnn8dOoy5HLZIe8mYdirUFNI6a0Qu5YUzqRy/BmYwc7DchFBa3GzrHF8fBsIg7l/7I1NQ0bjx1CqdvuUVJlYjh47r83M72GlYvncPb3/3PcP+n78edb7pXBX6tesMWeWglReZMmXOpHcl/TvlSalh+gKlxIYb8zMDoTBEi8omocZjgiKcbkFYfxZBD80+4QfVMJC24phDsyhwFMQg3vYFmpn7xA9+TCIhPBihmWQJEN9/LdrSjzdBzNxIrV/VleIeUfDkkeaRdBXECaZyZCJia24NuUsSpW+6SNy4MmA816GNlZRVffvQrePXVV9Go1XVN2mYLxQzgtwW1laMW4WLzRS1iEmsPPVLd/n6S+cY/GzYw3isChvLmNE/GvEwPWVxYwVS1iltuuQWnTp0aZfc4ofXaOlYvnsPdb/46vPLyqzh2/U2y2TQtlrbkeI3kwBeflTl5YeacI3rVjoFHrK9lF2c9IyxD8XmAJq6OhRYWC2hRZauuwoTF5sTSzj4tUtkULoOxeyq62N3ZKaR+6QPflyhWywJDJh6YRRrS1hhFKQj7uyGRTbAyQp7jNpaG2fRR2pDFe4UK0vkqbr37rQIWRLYf9PHZBx/AU089iWa9MWJNWrxrFZ0Kl9xWxWLbw9kuEanPvW89rDMzYzEJqkilxxZ3Idjd2TZ2qVenKvNnyzkbIsg5IaBx04034fbbb8fO6hWsLl3AqZtvQa5YRaFcVdIj8TqrkTlIGS1bfgSdUa6E72gOWz7JWHgU8KuhjtSNxgW0/IFlBM2AkZJlSBsdM1HFXJOEuFui1lBN2/l0DFmk6MLxyz/3/oQDK5XzSDn91x6YWbCWFps7ke+PhAM/Ssg0dlxUUHCHh0dN9d5Psjh7cQXf9h3fJ/L9o08/g8cefwxXl68YgDJWSx1o2jh8GQscO9cEjjvbfIRQ7UNpZ+On0QSxIsScGtMMAlrGXiEUIUghWJaZM3iSU6a8fS6DifIEKqUK9i/M4NSNN+PW2+8UM1aOnlivu4wUwqaMDOhAEZMWS5Z2WaQI2wzyNZzRqw3j5BAurmWwGN6akFD70L5TG3EjjFBGpmhJn/Y5ZMREDSyOn7Sikys4D4Fs/uSP/9ukpKJwMk4oUgPk6FJ5WQztIyU0EhvipzG0cIaJr7iQLKnYtNVqK8eayeHVy1t45zf+n/jkpz+F8+cuaCe3O1TpVpyuHUYO1oi44EkT7TjPJXsFRnjd8uG1K6nGBhh4sZyx12yhtcjK8VqJsNlHI7jF38eFaFybjAtHwKb58gQI1jA+J4tmfmYex6+5BtccPmDeL3qkfouuJIFNzLHV7vTiwVjgKPYzgQzv2ahFgmY7lsAJuJNzTY89dr9COdaBZ4NGxXsa8ZGOXEC8xrBJI0XYlvyBX//Vn0zajQYmq+Sb9QxtoipKvG56wNJQBu4GBngkotooedJEZ+QtkqFhD6b0Jx2GXBk7/RKefv5ZrG1uIDUw4iCxbNpk2maFcz7rsYBhm2PhQtWG6chI4o0LpyyYCmK4iJT0XY41d7+WX3YuhVTGhGfcnsf3sdvHfYBIJ3Lxc1TtBZL3c0bu4KISfi2X5eFP5LK47fQNmJmwShBqiBFU6hUZdLgshbtrPhgDBz4fwEqMyWrJrALGVLz5TwRvbOGNI9DvGRaiOfDUcrBc+DMxc23WD/3mB5LN7XVMVSYsC6UkeQqH9h/Bvn17MDU1o52aLVWMJeElran00PK+nabiPe5WOhgE8pP+EINCFc+/chYvv/yyUpO0J60mHTDzsBV6yNu23Rn2OB6Uv1eO2RhyI0+aP4loPyq8J2Y8MJanY+KBfAnpc7LguJMW34f61jXdU9+140b0I0TJF/EDZIj/M+WbR67AxFBJDpbsvfyeDMrFKrKpIfbNVnDztddKEzDC6QtYoa9jzQqIVyszSIoVee6OM3Ac0nhjPooVRXhRorho1q4EKdvhUTYdqePYHBIW2vVg5Xz6H/4k6XaZ5aIt6WN1dVWkAuKvlCLaHbryzIpJUl18xIPOpOTFmlonamRgQJLL4eJmGy+9+KKcLg6e3mGzaYjPSK0ZlVrvsV1kYU+kN7ngI+ryWDWE/C7PiZvN4mJzZB5aOcGBJsfE3VKioSliYcMsjNvzEDZG/0aiMEdIi6SEQxHFUkVZQC4UVaS0U8YBGAqiV8jksmkUc1nMVSq45aaTgobTXpJLZyvoybLPo1IdY+2qqsRLltR1watCtEPdQeYGi9DLtoQ5hTJhgp4jXrcwL/UXf/RLSqdQCsx+GrbLeqSwlLcAACAASURBVGVKEFWFpQB366t5MzpYVD9cSEuRplApl5CvLqJXrOCVl7+K7Z1tT/dZxobCwCR/qGsuWDgY8RASHKFK9PAt8xYPZ7nrFLIeUlAABfprt7CyMoMBQ5mITp1HF5LOz47b43FPPDJc4dD1B8zpm2PFCSSOzs8TFqbJylcqUum5gvVqSWjC+kaUVIHgwHqqsFxI8zrsygGeLGXx7ne8HSxl5D1VvizqtFWrBpUrtJIxTswkBMxqxY6SeOcAmh/i0qy/8dmiPs1dFqR+4xd+ILHuOlbiQlBBXQdy5FSToGDeLKmzQqpUOG/0YpHbvc0EXaFBfhKl/dfiqYc/j3q7hW6LjpgJCz9HDjZBei6MFtE5zrHrAgkL7jYHH4BNCIF2WYQXopsx+LTnlKOUIZ7kxQgeesX1YyG/NpwLTRM73cIWCwNDy1CdcxMYPFxEkiNzp4wkYzufQsD38FqCdj3lmvI0roiVFM52C1tXL+H2G6/DO9/5Ts/W2diJZ/Mlb97JFRKUsZKrCKtIkmDVjsHYHoV4XxjLqRv3PIAcRQS/9cs/rG1n5D9ic27nvPoiiuRMzbgO99KfiANbrR0MhxnsP/12/N3f/SUyDnZQOxiNyJiTzDoZB4w/m80Sb83VdYRtob7DBsm++w4Zt62pUH9qCUVfg8O3/HHs4PAFIqQLJ2/cRxjH2GMMDKG0WxyNE1qo3LLVUTHTx8RPJl9Chg4se9Kwhj2VQb1hiR9OGGu4FF4hjXTSQ7NeR7u2iU5tE//ym78JJ48ftbptItxO+DAGi5mRICMGrs4oRxx4gkwwGFUl6iRDiMpkcxuVNJFdUzLlv37wP2ixVZfsZD05JE67FewmgMOACM5vgP02EH4uwczR2/DYc1/F6tIr9neVsUTLJ7NrDCcaDcKmJDdSEMx+M24OdR12VWqIVZNy4v7/VYzane5lWu2MIUtc7FDX4Wz972x0/C7s9bizpmuz84SXB+k6LlhRCWI8vDzSuRISpRfJiSvK8TThNAezXGE+voE+bWmvo2Cwtn4VrfqWHLef+g8/aowez9eP8geROxBl2KBYsW2UhevLUMlNUbxOyNXyF7wW7z1OqwoMI/WhX/mhJBZUgIX3BIv6qmBXWALe0pPuH5tXyf+dFvLH34L7P/a3SIYNDZxMC8F3TMnxMwJDDPK02m4Lk0wN79rmcFSsPHfXWePYYkxRQWnjME63TJbHcKGmww+I3bp7bbNv8dz83jJ4RpDQriSvzZEv+QxU105CMNvpoU62YOYuV0A6V0QhVxSIwQVniljz0++jTnIGG24NE2ytLmN7ZxXpwRA/+1M/6R0d6MgydUmVbpskiBARchl2bhiZxeduucliCQfWKckjs0aNOCTjN4/Ub/3iv08YQrCaIfhhu2GPYa8RAoUDZ5JvO55aodnroDZ5E557+CHUayvyUoOcR+FhJ0LtdudHEVMW0N8xcgFDMKk6955t4i15Eeo7FkEL57zvWLyAH9NZW0Q5bWMtu8a97XD2wqEZQZtj8Kny7EwFEqgcYdVWshTqn0V0NqHuw5C/njMiZrqQQy5rxREZr4ztscojGQgf315dRr2xjnwqg//4Yz/ila1dLSQXJgoNZJfFErW+K9FKLNp1EBs3pMyRNufnGZpsXj2/mgYGUh/8T9+nKk5WPoSBskm3zJDZM8szx1dzZAylYrhEqtLmxLV49itfRLOxpsExqWDCYzsyYL4g9wVRn5+ntgjnKHZbnoUEASOSOapWGUZb4kv23MEVLTpBBu4cx8/HwZH4Pr4K2Bgj/MeCh6NmKt18F4Ieso8Ou45/TuPwWD6XLig0Yx6/n5D4UGLnS5RLJEZah0JmyQrZNDZXCRevo5jJ4Sd++AcdLbPuipayNAdTIIwDMOGoKUHkfsS4mQptFlrMwBbWirtW5dxxsWUPnPX5tZ5qEP/dr3fyn4Hz2o3suNDpY/KGd+Lxzz+AixdeRNY9VO5wMk0M6SJD1CoUgjhnHja9cgM1DB40ocupoJBCZa42Q6qAT0cPOQb6K+4nNjDWqoPPFQscKjoctPHnDOctBM5UqAmVFbfbDhnVTHmZrqIRvx93eIoOWybHDJChXKRZFyc1hiafvdVGIZfG9toyavUNlHJ5/NSP/ahrNIIO1Epm7zkHyi94nbnh6bYfd5MlZsi4uagNhNx5HkB22pHMqC9P/ebPvz/hgKluwhGKna3p9fAodpOBdmzlZIxKJgJanT5Ofv2343P/9ABeefZRZNJUw6wVtvJdAhGhsg0T52TKuzDKMLsVhN11hEwqyEOvcDYi2c8HkkMXjXr4wKL5WLw5WgDPzH2tGh/f9eO7elfr2K6WgIAolJVARdGinM+BJzBYo6XSHysglLOWNgHJ5stC3bhjudDKQPXbqG2to1nbUi79R37g+1+jrYLepDVx51g5ctcsMUYrLdrtLxsmRqGqGEAUxF1QSprhN37ue9VAx+LBcFJMYsxT3m2foR3mHYXDzhK9ajVauO6d34Gnn3gWzz/xJXQ77NhgHuHkpBXDGxZuVRoR+1kmJ6V8dixQ5K3lhHmMKiKe57HNSfOiAW8UQGecjk/kt83W72a75FX/bwraQ+XLprmDE9/H5JFLxvdxh4emkJD3jDOnZxqShWPv0SKl89o8SOeQVTtN443xvflsVqyXTquOublZfO93faelI51PF4Idv4tx8e/jYwuTE8JhPpDVltNB5L2ClxDzl/qVD/w7lexavbEjVGNNVqN6kQ8RN+CFFhYWwBYQxWIeSSaHzuQJnLu8ise/8KAexpy6IeYXZ71wwOyWhVKmqqimVNM84lPvdn+IQgOOje0raYMCD4/sFheedj0ctkhphoqORY5F3Q0jvZPDGGWY4+JzRQgY6jBaXkdnhQA4ct5zRmgZm+8RIVSM7w1o046sSWPSnzVGSqrLxj/b4udff/11+OEf/EFfbGO2hJNq/lHAqJ5p9HZlaTmHDDONYxa1cdS6mltH56h9ogpUc/BLP/OdymczbolYkzsnVGXknMnbYq8RPvSo1ssTCCwZquX24NIO8MTnP4Mrly+OgILyBInwjEENFQpEzXZL3hrTpq2nWBD+xu1sOGJmUkIhW2Jf2ACT/DExY4iZdp+XvgYuEJM5vtPDHkc0EL5DaAIrKjRGy8jR89BHvVy8dZeySwlZKabOuU4K1cQxy6g0R/dXjqAuuPRd73o3/vk3vHdMjTMnb+2/FPJGaOpOqXnf5mkr7aww2Xh9Rllwe27fjHiC8WypX/zpf5swSJeKYTG351S5uATuc85bjpCF8bEe2u1jmlNNzzFVwvnuNB556LO48NWXkMomyInUDiwszo2AFAvx0t5vu6ydHdpDu9ix8NiNoY7DpBAXd1/JAIxUImGx1N5uY55Q5fE1JinEJa7Pn2PXCuN3vH40qeS5ec45FtxqoS29Glg2+WEquqcL7tGCqWAjTrCXaTTwEVU6ncKHPvQhlUiHmRPbhw7pWBp2V0CtBp73NQ3rFC0nMHCiJdzeL2a0+B45aSwf+In/OyFXiv27SbpXB6IRMS9tOLSyLN7wLpIQUYutBu9ZdIcJznXm8ORXHsa5l55Ft99GOrHWUlNTE1LZFDcurrzMPqE9a0jL3msGtJiHHwAHB8hdoqY3rE5UV0Dz3G3X7qpxg3stsRI7OhY6zAavN55wGXfUYnF31WhMqoFIRtm1/IBSvS41I+dJZLY0uh0nGoYdbvdUkkP1ru5L0XigVMQHP/hBoYCGVnr1ihMTuKjGOHGKkYeD+tmTM0ZiMAatSIteVGkIk7FUhcwpu5hC6o9/9/9J1HzVS2eEgdDekBJM58JPGMhmmOVJI3EUiQsshIv9vAg2II2vrnbxwvPP4qlHviSCvvBqVmeW2LzVPPKYVLOPhhoV8+wRYrxyld96OBOLEwLAWnH+jTtZsbtHBru7w9E9j+3Gw6zxRRy/7tdqgLh3CA0xcj4rd4xahgRI4YsgJ4222Om84deElookje1QFjQaF+/EyWvwH37sx91OBxXZulOpfwrDWmbt1FLL1HIIp1KqhRyGHWeiOOql4zjU9M+aBFohgiGRCls/9td/mBTLRWTUSwQCBZKEKTfr2zGi73oFQ3qw60QpNEmxwRtj3DSu1od48atn8ehDD2B1ZWmUiy6W8ihPGJPFvHEvuAtb64sbPkOYknEHSw/oD0xvM4SGYyTGzOvGZHxtDB3OllKKXgfN7yMBIgFyGz+uBew6VuhOSFRC5zy34I0x2aNIIW190MI+mgOaRTIIO2u5ezstIY1f//VfwczU9AhsspbfFs4JKQvbzHvGbg/AhbaakYznrpW/GrP1u2RM3ziujVMPff5+IX9q0KL2y757vGwm3H2Lei0nPY4hy6HxdFo/yeHxVy7jSw/8Iy6++qKpmEwa+VxWhQfRp4XccF5OdUjFDLpt6xca6pkTHs1aaU85iVTz47tw3KabJTPHJUKRWPiv1RKx2/lc4/cct7OKSZ0gEOxPYeXBb1NDH2eQuhYZjzLsnhmFWeY505QbCklG7Xd/93fjDW94nXPw9FcRMGge4h7RrYmXFzVpnA3rfPQe07DUKS64chIpcKo5G8rsGcnRk1kPP/JgQk/R0pykYxqYMALhnWLbb1uXWz6keeNx8k5KD8JS3VyuhOcuruIrX3wQLz39+AgUoNQyfjS8mXnznpAhkeDTAyR9CxnGqzPi4aJOy0AZE7RQw5EsYYO+r0XG4vOhHcIPCDX7tSp+3L6H4IzfS8wVz+Pzmv2ehakhMCEs0cFR3HkdTZHHgYMH8KZ77sGdd95h+RWRRUwTRe6BZkkOn0cQ0UslFt9Ewtil9PLDWbOMJVG0XWbqeMtt81E8qfT5z9+fsBMv7aHVPRmfigNSAl0XIqmcRXQseLOeXqxgZH5a2DbhTZ2pUcCVtW18+nOfw/NPPKLUpXUpsm75LMfhBLJVRKdjvcJZE8XidoUT8jDNQYtJCE95F3TZ7T8mQqEcOscH8plRV4TAv3fBEXOc+IpESahsmYgxtC3MQGiPuHcsfpiC2P1a9HYfe/fuxfu///2iHhsM5Pdy+rAEMG3PZxTh3TGxr7uIEuwU6Y3reV+WRRlgYk2AeS91qnAiYtC2rJWJbRoCQcIlIivorcVSD372kwmzVjqRJ2vdh1l7FQDEoGt4axSuST2pgsT7blLd+SEtjDFT6QKefOUM7v/E36Fe2xoxIwnAWO/SrOq2u11SZ62WizaXLzEyHXCJiYoJjh0+PtFy1EZJGh65YDZzHIXiIkZIFRBo7HK+N8xULGjYXA1ojIgYAjCeJ45dd8cdd+DffNu3e67AKjZpQ6PG21SpF+2JXGmYugmZVW8QhwgnkjtcvD0nDHLhtHO9k4L5GAyTdxeVi22JKzp0Rhahn0EBoGoX+vfpf/ibJM3QqdPWLstn85icncYLzz6FYcIwjJBnFXv37ZHtaNU3MUgySGVYrZlHZgDkK2wIYwxPqphXlrfw9x/9G6wuLwlDZ5E4ww+q6Xqt7g3r2BfNeoMOKInOlFEI70kRIy8ECXG3VktxtZzH6LliNnZ0ksAYOTGw5JjIWAC+N6jIdoSUYf29riF8/G9CbdpGCQ5f/NAEHCfr2n7mJ39KY2ZhgHqjD/qqTbfEhqVbWYynpvYD48rzFa1GuLBEIlUbzoZ9Y3kBnVDk7SrDbBCNMzqxaYg0mUHhs+ikBeMPcvz0j4zFk0Lqr/78D5Lq9Ax63bYkgdX611x7Eg/d/wkcP3EKi/sO4+WXX0Q+m8aBw0fx8tOP4/ipm3DxygomJyZw6dXnkJ+YQc/JJCwiT+XzuLzVwSMPfUYdE4kzVCtV84QdoCB0yvBASJDiCqtdGn+Zat/9XahNBXoKKSJDZHlmkiNjUUMtj9vmXe+eMazVnekeHpoY08N7sPjC8prjsWqo0sgw/b8/87OYqU6pw7HUvldi8Hk4FoavfFajEVGT2PtCg9gzMS9hVCRRmdzzj0NtKDChUaTxmPpVBMDuzz2rvuUpB+xVquY6lofv+r34GYFVH/nw/0hm5mbVe2t6egoXzp3DnXe/Dl/8p0+qo++RU7dgmcXvVy/h+tN34IXnnsDJ625Coz3EwsIcHn3gozhx+s0oqEVFHfv278fTX7of5cM34S8+/GEsXVpCPp9RO6geC/ac6cLJ4aFkQnpiQcc93rGFJl4VvTsNVCHQE0wWS4wYkGKCQVNjDppXcnqXYOamJQyBKbN6xc/90G7lzus6Bz1Sq9EiOrEMHR1F64OSYHJqGj/3sz+npEh446ERgnI1KgOWX8IerB3tYIJNpkms0Q0PYlPNupMuIoyjsLIxACneuXzBKkM8VCQMbfQuo25Rm/R40kGpKN+l06xbXThbpdCGs/PC3MI8dra3MT+/gLOvfhU3n74Vzz/5KNqNbVx7+xsx7PZx5sUnceTkDUpyFEtVzC4eQnlyAk9+7mOYmN2L/Ueu02IfO3YUjz7wcUzuO4LOsICP/t1HUaMq8dZV9DKFJMkeGUU2asis04QdTmbVIl5HNebIjHunEarJ3ku1pcSQMTVoFY2aPDXX3c1ta4d7VYWS+4RMM1YjxYlnSMjvdz16i5F5P3rXFk7mVaX5rne+Gwf37hsldsLBJFeNY1LbixZPTjCba9i4naQQfk803+NX7sDwJaiGubhsTBC+C7/yOjqZIA1t0si9B6N0e3vHyCNk/uq4Spbx9pD664/8fjIzO6u2FWxNwSTG8ZPX4crFC1i7/CoOXH8bFucW8NzjX0B5eg6TlUnUG01cc/I00rkMnvvypzTA46ffpAXau/8AXnziATRrNRw59UbMLsxic2MLTz76EL789BksXb6sXWGevrMynMkSB4lG191oWZl4q0h+jhQqPgiPfeAujxYUVu/sPcZGoIsd8Cq1SJUfdc1OiJQqde+fAIXh60Md+CoMWiR9o/bypTiYcbP4vEAubQ1riO2Hz3H06FHccMONygqye1TUG/EZFNuzOW+vp13ISwVMSgRRi+LnpfCrteMsqgcMhZj1d1w0CZu34OTOpkIzSDnB7MysasXYnSoO4su62Uj99V/+j4TF6LWdOqqTVaxeXcbhoyewvbmGK2efw+yBa3H0+LV48ckvoj8E9u87iq3aNvYdOI7iRBlfffJzaOxs4/ANd6HEHT87iwuvPouNy69i7vAp7D98rR7wxScfwKByAB/72Mdw+fKyqb2BdTgO+0Xpj7CEoQapwnzIyLZx8Ny1Ukm0/Q5YyJN2gbFsmLXVjOI4LZYxHV6T16ZajyTQbjLFD5rLG7NVbBSP7y0c9DCR2kQcNW8G7zn3cNCII3CcLHZg/7SJsp1lwrCM5nHYbSmKoa9jdKs0+sMu7Y4EgYe55Qs2N9T/1g/V6r7Y+ULOGokjjZqKKNVpiTVfbPbXrKPJDlM6Xbfgba0HSP35n/5uwqpEa59cBM+Xmp1flId86ZXnUJpawPEbbsH5l55Rw/mFPYfEpZqc2YuFxUWce/ExbK1cxsTiMezZd1iLvXzxPNYvP4t0YQLX3vI2dSB89bkvoNnq4vMvLeP5xx8fqR9BmNHPVOwV271c5JKfFMDfaZFzu0kaIWV+Qq86D3i2R4APTxQKh8lLYwngMOHCtKrRjiyhEWaBqcoAddQtSr3COXF2hgfbVZl9NB+DZT8sMOQiqZuTzibxhgEOdFBQeF/ZVPfCC/kSDh44iONH9mNl+SoOHTupnnArK1dRmShhdfmiHK3DR67BytUVnXaYKxZVhdlt1sVJLzAbmStg2GubZnNIt1CqamytTgvVShkNP6lPWolz9Vd/9jtJvkxyoDVutzjVmrGtXDwnZujJG2/F8tIFbK0sY2ZxrwSjOr2gU/GuXjqLnaUzQLGKhYPXYnZ2Adubq1h69REMBykcOf1mdUQ899LjaO9sYjs7j4985K9Q11FN5pUyZOFXWtp9+/Yr3hYzxI8nZlTGn6lo1ZMz2l97VaaFFlSnFk7xWlJvcaY2QaOx46oihqeaFN3XF5+2UPdxhzHUvFKq7jCypo0aYZzUEeDLOFizGzNb7xQV5jmGoNjeyZgEnt56772YmpyS8DY2LmNicg7XnLwJly+fxc76KvYcPIyt1VVkEx4ydxUz+49jbn4R68vn0ajtoFouQIfjFLhBymh3Gug0a+i1TdAIdnE+Un/xJ/8lId+Z+LUC+X5f9pDhQH19BcNUGvsOn1B/tPUrl5EpltUMNpUpYe/ePdhYX8ba2efFtZo7eB0W9hzAsN/Buee/qCMo9p28HYcOn8CVSy9j+/IZJOVF/PnH78eFM+fQ7Rnezfvu3bcfh09ci/m5eeRy1sEvuv30O9bnrMQDYZx2LBXrP3Px5HQZqXrk8Qu8oPCy+I5xrjea5zPy89FFOECX8URKNKoNgYmkCSnBStHGkY9RPDiWw+Z4IlY3xGs3JByhdrLhPF/T4F8ybCmQxw7OYX7vIdz9unuwvrKEKxfPYe+hw6htbKDb3NKc7T16E0rVKVw5/zLQazGzquKLfGUGM/OL2NlclZlg10rejzSpEos1//T3fzkR31nF3XYqnzrRF/LoNJuC6fbsPyJbsaZMFoeWRbZYxsL8HkFzK+eeV0gxufcYFvcfE3l96dXHsbO5ganFAzh6/BbU6ptYeuUZtb185lIT93/606jvbKDR6eOHfuKnUW8P0B9aX/B+t62meYwfCXiwebwWiIiR0CnGqhazdhjX09apM7E1j+VxVRFeqcpFaUMrciAwRE1g6VaDaMPTDR5XcMnioNnIkAmNU7WqMWIDsKHNpcPJ8NLOFfXTdrx8KFp18/ddnnnqfcfl7XtmXGeSqZdMTxSmQwcP4Z7X3Yna5oaAm15vRwvOse+95laZ3NrmEmqbV9H1as7yzF6kszwQponWzgpSgz62eYpvZRKTc3uQ+uPf+/kknS2gQM/RWQ18eC5Kp832WAkmpxcUpNNpo//KTZUrTmDf3gMCA66cfQHDfhPpyjwOHL4OxXwJaxdfwtrVcyhOT+PaU2/ULl8+/6zUYbtyBL/727+NlbU1fNcP/LjKaLa260ilzYwQwKF3WSa/LUlEqqCw8RpimGZJY2L/MaYQ+xh2efRCH722N9cbU8uWGrXr2kIbYNwmsqdG+EaJChiWX62Az1pYRIYvgI02QxgnSQaiJWqSw7KMcdXbTYV90aXJEiZ23rbF/vZ9HMhqHRSkPVRTwTH1UC0V8N6vvw95HajXQnNnW4zUvcdulTlbXzmP+tZVdFtNadvS9B6Z1+3NDaBXw9ryZWvik6RQnV1E6g9/62cSNpnLuo1MeUaF8KBaMOoQlylkeUh3r42GmCZZtdCYmJyRyqfdbuysI5cvYe/hU4JXV69exOblV8XeYAjGU9uvnHse9Z1VzB64Dn/2N5/EiVM3Y3pxn45n1IEvLEFVKGPg/wghEzrURSGbt3M1szxkhXGmgShpgjE89LxnXYLZs7TXZN6YkGRXNdGKad37p9dPDRKN9tSvLE+wYjCCcFlxysW26CCl7gahBfg7zoslM6xsmDvbnD5r6MfFEA7gvcKjC4Oa0PF0AF7DY2p+r2ILfc5r5HrWFLA6kcc3vOPt6LcaGPa7SJcncOyaWzBIp7B+5Ry2rlxgcY5M4fzB61EqTmCYdFDbWMba1SWFqRSwyvQCUn/wwf+YkKhAiaItYvsIhhNsXqf2Dil6x1UZeXYopoqU9BdLKFen5KVurS+hV6/JBMzuP475hUX1DVu/8JIWYM+J27G4cABXzjyPVnML5YlpPLvcRXlmDp2etd8S89QXkhk224l+aqA7TMzMyXazl6p77oasWSUoEyqceDaHS3kbCi4YPVnZzYT/DeumqdFB65HedWKAWlzJy/YjLbwgYChTMlCOOrSAOYK77BtpAbD7RFvevPkJ1pGY17TkhrUXCdqQBMd9iPBfDDJmVScPaAW+5Rvfi/SgZ+ZtagYHDl6PHoZYv3IejbUr6LGWPJNBdeGYmgT3ei1sXL2IAR01xuoTFZSn5pD6g1/70YROGNtIkFrERVZK06sp1JvDKx0M+7W0W5LKYnJ6CplcEd1WDTsbqzqFoDp/AAcOHlEP1NXzz7PfFqb2X4vZvfuxvXYVm8vn1PZyYt9NuLTdwOb6ttAuJUl27LhFmgp77Ta5s7DL6sO5s4lghSMU5bWMyyWILhQcL71QCpESFd6ey0piTCtQGFhTpSMn/WgK4eXMoHmKUhAoETcJgZU80RsPx5Dawzh1LHw0UkR49LxnOHcBgYawBFrGnyk00gxjPVzlHWWzeM+9b0C1lLPqmvwk9h44KlOyevkVNLau2rNkM6jOHQZDO4ZrO5uX0anXrCd8Lo+JyWmk/tsvfH/CKgZCRTlWIFKUrNLLzqygM5GyKkURERkzisGWQ5GdFgoTGPSaaNW20Go0QCeBi02MdvX8CwoBJhaO4NCx42g2a1i9+AobV6By4HpcqvWwvr5lZaaqELWJ4iIrJednafG+ERLxIQmSiEbknCum9Pi5qNfm7jOWqhMTiaDpyGg7tkH88yGUk9fnlIywMLA7sG4S2ZQVshMjUNJDXYzICvW0qHvhhoFbXpq7qOskD2kYp2AFeV+dFb6mTCcSKiGMwaAJX4Ff3/2W12P/4qzWZXrxKKbmFiVcq5dfRae2au23CnlMzh9BuWTtvzdWz4JUETmZ6Swq0zNIfeg/fXcigqHjyAmbzbK7AltLyzYzCc4qA3c2VFCQIJPn+ZhF2XpOXmN7045xqlaxsO+ornHlwsvoNtaQKc7iwPEbJCjrV86i3+mjtHgMm/2iuFRXr1wxRMhPD7BeXl0hZOEpR1ZMRx555YUQLSpELz5Uk9eoBGU9eJ4q11RmxOKWnuTCkCnCyfDzNpyDprM0WJbkvdA73ThegpSfFnLUbqQww05D4PUUQXS6fta3lSSHLQ8nLnZ34O2RJo0jKFyVuYDasVFxxOV77nsD9sxO6muDMwAAIABJREFUSkUX5w5g3+IBLeLm1bOobSxZGXRviPk9R1GZmsH21ibQ21I0pANwGx39PvVbP/sd1AFyoDgwNokXu8MdDJaeplM5JDnLVVN9m9NCmnAJ7A+mZCNVx9YWUrk8Fg8eEzy4fPEVNLeuIElP4NgN7kEunUW31UV25iBa2WnVSa0sL2uRGA9zt6lGKTPEsD806JBN5ssT4IlEskHecC8otOwWQc+a0Kd2ijxj8uDN+7bOidYWK5L+dK7YYpMTpaSHs2aiSWyUNxGv5vENwx6dKPY86arUNpoXtPtdMw/eKIj4dajigIEjPx8xdhAX6DyFoxhCbQ1sR2WaEuy3vek2LXapNIGpfddgbnpBuYzNlbMYtLcUmRQmJjE1sx/FiSo67SZWll5B3rVVNlfEgIWHH/rAdyZiOaQtO5RmGwmiUZ6xIQKsGmVWJqZTVmzOXaiOPEWUJspuuwaob22LZTo9u4Dq3CK21y6jvrksFHnx0CmUKhWsXTmPZn0HufIc2qX9SkRs7WwpyU71yyOQAokKtRyn+ubyhosTdaKNJVOTqUL5QGOlM2Ez6UOojIZwqx+uqkn1BjTMGFEzWJ8XClZeuLLial88xqqETOkEqTmfU5iUVnXnyrxpO4SdziCzXJEAEVbujFad3R1HZYjM4Od8e8M6TmQc16gx+CE0//xdb0KF53snKew7dBIL83sl1Mvnn0ONNps59HQWE7P7VRde21lDNunIBxLUW5kStzD1X372OxOzOVb0zZBLaFTBHDX2CleaMLFQQkcTqNk5Y/Gy7IF1sx+q9zYHWChXMLfvIHrNbaxcflU2ZfHIDZiZWcT2+pL6irAJfXfqGvkKXGweDcFqTsbtUaHoLbSlVjmZhFE5JmLcUc9katGQNf7nwgX9iMQJ29nBJPXKEYV5u6fvMU896HfkeCrP7nGwbDeb1PJ0wFJeKBfrzsLDVt83liA7kKJkhjtYTGTQOYquhMYPYzLeqFfRwcJy7pGPtwaC8iGcEcr+qd/yjW9DliatWMb8PvO4eZrP1sqrqG+tWPuNdA5z+46qgrTZ2EK7tqbjP3QC4YB14hWkfutnvt11hpXQBhtEh6MzvFExALnZWaTzVn8sJiSTD7Tn5K3xZKC8nYqrcy1KE5if36sdtXb5FbFVJvccxszcgjr4s3mMSIvlEwpVOmxDUa/LuYlcbuDVlvWx8ETd/dkf1Q84CcZKwkXgJDsi1uq27TQgr57kLlVhuoTaGTHe2sPOv+buMz67cs6eCrW4Oiv8nCRJOX19rzrReR5RgUJBs8pSMkeiEQl3KtOl7CYch89F01i69jI3znc3X4MttqzDAgWHWmeyMoH3vO1OTFan0RoMcejoKVQmJrFT28L60lfR7zYFnKTSZWlT9UEb9pB0G1hauiRNUixPYDhII/WbP/2vTY37ohqldRdW1NmWKo/M0OCpFFUYsnho1geMks42URaCMITIozI5h8rkJJbOP492s4nKwkHMzC5qR+6sLVviYvpa9NgxMWV8rJ4X64fHysmXSiY1iBAn04I6e9MSGNwd3Fl0jnhdlsFGaSwFNc77oAqLuF2qUud/GeOFcTX/RuFmbRuJAqq58lBqBIl6fM2TiMPmmrnY7aYcp/Ba41w3LXQO++yVZJTrqLSMggdreGMLLSrx6IjqtDTD1FQV/8c736S5nZxbxNTsfoVXPDu7sXEJnXZNglyd2oPK7KLYNIxqCKrwpGSmr3fqdZRLk9zZ36Fi/MjcREDPiVD44+CCtX5iC1s/c1pnhDA+ZjuJtJrCMUHP9BxDNoIwk/ML2GKXgc01ZAtF7D10UiqPP7MNZmX/ddjqG57MhHuj6Uc9DW0RR6GKdiorTzpIuEu7hpUTEVP7KLbS9J7oXLxI6PBZomCdpkjtuHg3jdvqrWk+goIbTQLkoHq7jvGwyey9dX7UGVrcJN4dOUgQ/MoIYLz/anjaUZAoCpXrU+5sgwGN2B9IG1uAc17vufs0juxbtM2RLePwsetFaNje2cTm1XPotWqoN9uYXdiPdHZCm6DXb2NjdUmhqDUw4Jrlkfq1n/y/VJ8ttTFWlmq4MGucrMsfU53y1kX5zWHo3QJ1oEqprF1ON39re0tYNosGipOzysisLZ1DtlDC/P6junnS62Fnex2Ti4exmSygM+Ahbzy1hhMPdFpNLabSrCsrQsbUUbHfwvbahtSikKiehU089ti47XZS4Hi1pdGS/MSByIJleaotbbkVHhi4stulwPhscYCLV0+6lpFH7WQ/2d047H3sFEE7etF4YSE0VmCw26dVrFvaZTpq6pC4W8BHLcCzWk7fcho3nziMTqsmBK5QncUij+FImGhpY3PlPHrNGjvJoDqziInKnO7RaO6g19rRQQHUVKRIsX9b6hd+9F8RNbbzPoTC++GnnguWeo/KSTVbpUfMHizehsIPbGOF8GR1Uk1pq1PTlldOpTAzN4+rF8+jN+xg76HrpHImiadfWcLk7CLWM3tF9WFMScePue0aKTU6M2tTCRFmgsjk5RENje0dqXvBlElw2g1vHq9uDApSLLx2ZZza5+UycVipOh6JyMIODFGf6ScI+yLuxskegqrbgrFbuctD3ZN9kuJCC//uW6/vsb7qTGqIaDFioBikGqzVfDaDt977Nhw5ehS5BNjavKjsI9X9/IETmJyeQ2o4lBrfuHpOY6YWzZd4tGNFgkuKdrOxiWG3Y4fJcjMih9Sbbj2U3H76JuxZnEW5wGMgbGcYsmTHOUnL+JlVVNuSfB4xIftt8CV42MpE2equqxXtNDam3X/oEFaXltDpt7D/AFG0JiqTU9hcX0OhmMdw6jp0kBOjIzhZdNSIVtG2Moxpt5totWroNNtqkcm/G1drt8JDp+xSCBMoHAv4MXaptFLWIFYdqRB9x7UQdppwf2AkiqhBD7ttTiNtOyfDW2RFoTyv56Wz0jKEPcWMTsk5ox7ghomW21UeLyV2ib2OHz2Kd73rnTrakX7H8089La0wOTcrz7+2eRk7W5tqaLD/6CkU6FUnJG3WsL58Fjwsjru2VJkBUkZy5GIPBy0Mve1GVwfDVZC65YYDyc52DZ1uH3vnp7BvYdKci2Qg7teeuTmxKKpVghpMORpRwFgtwqasFbPjuJwoeucKHZIheEYlJW91dQULe/ag3e6iPDktQiL9vurCYaxiHgl3sLJUHaUtZZO7jFlbaDUbqO1s6G+M5UmOCOyZE0Shi1NpFaOn2bynjEabJTNZxc/WoZ+JClOlPG6AgsoiCNavjRIgsJpoU+27rUWCjCDVOxiiFGd48z00H96TLCNUz2JrhWR+AnAqm0elmMVEtYiDC3tx/fU36Pip8ClUxpMCnnj0EQlloVpFv9XC1tplgGeDF4ooLxwWKbRR20aztYN2bUtzRH8qW6yiVK7aCcHtJrrtJhKCQATApE2ySH3vv7o3YTqvR8eDXYa9+ZyqCr0/mb7qRAErLdGBLf2hFnl6ahJ79u7RQSqGaLGSgtUQrGe2Qv04TqJa5Yl5fRQqVSFOxL6LE5PoVo+h1UuBNWeKibsdLQ4dL8boGxtrGrg87xbP/zLcOcJEqWOPkYm4EeUSEZD1awXrrM+QjQfAqgyHKFjBCIUsT2ZhgEgDNGEeOAU3OxbZ4E1r0MvPTfL0PyJnLhhWnsPr28HqFMZKtYo98wuyvRN54hCb6LR64gIUJmZxww03jLo+EKmjKfvyF76AieokSpOTWuy15fNqbstoZ/bQtfrabtaxvrGiEJbRMdkz1akF7XpD69qq8GFYxnFIjdP3+vkf+iZtEjZmV6rNCXW0wZwk4b7qprRbtald5z1MlaPyqg4V+fnpPTOzM7j2uuvEqCAIYIOwDj4E7SNVqQashTkkU0f1WcbqFBR+JQOD8XOzuY1+u6OfyaYUB9pP9RXgIgDD2leJBOAn7vCe6YxVTPa7BF94CkBJlaOBgKnvJ59HqVbadfNfmC3Ty7NbnFUlJzy2Vh8G92tYp8Wdye4Kx48dU/NZ1p2RYXLoyDVoNxs498LjSPptEGsvTC6iNDGtkwXjUHoWPfL5udiV6pTCrPWVZdRWz9uclWew9+Bx45HvbIrlQ4iaY2r3eiiXp1Am7yCblT3vd5mOrqtdds6Zralf+YlvVehFhUz4Ubli5oVVAdGjhTJnw20UmV4CKFxN8fd2Gp1liSIG5c6k/TLbbwT9bsfO/5pfXJQ22L9/vzx3kh6Ge06LVkumZiQSqKLIrWq0ttDheZs847vZsF2tQ8GNzMAXcXsKJl+BSRND77Pdh0jypFsVBcwwNOFY5ZiNjk00Z288V82Ja+zU7JgI1rn5ATlk41II+PXUtdfhmmuuwebWGmZn5zAxUcX66jIaNfLF+rjx1rtECrx85ln0W3XNyfz+48gVyzh06JA0DL3xKGp89OGH1fF4Ye9BXL54Dq3NS1aDXZzGgaMnNY9rq8syZdnUAM1GU2dwZrLkBvoZpMOekk6N+rZiciat5KP815//ziSqIuwQUivoppo2NTeCeXczSqPOu+pY7b834ELagQkJP/vLSkkNmaOU8e+0pXSoKCjqMcJMenU/7nnft6Pf2UGjZWgWsd3hsCe8emdjw8kTLQmWtWvmrjWP02yxOZb8T4I+zzmhGTFP2QiJKrLzDglBPxpRguh3iOPmJ+QxqZKy9GppghqqjLfde69ds83zQbMoVytaTFasVqozow5Q3HV0Lq+/5Q70Wh1x6evbV6U5D5+4VZNPPjmdVDsdyMptv/DQQ5jU4Xd7sbWxgtrVc6i1apicP6bUMcda49mpTXaeaongQLw+V54VtVspzWSI7Y2r5tekmYqeMELGf/9F9kET3OMkPe/d4VxsoWVaLMNwhdCovYNpOU2hkhCEuaPO2tpRmJPDybfLqwGxeox6aa4awQzVpyWXTuPU130LtjpsoleX3SNEyd5xW5tb2FhdQTLoOH5uxEIuaqdDLNwiAnnebPQeDVr7xLG9/4rCoYHIlJEGDWhW2pr0q4nyqE6d5ufmm2/GwX3k0PdF0ZXjxRMH+fBeU85Qi1jC6soVHSBPUn5UuzS3N3HkhtO4dPY8Bt06NtcuCTy68dZ7sF3bxpEjR3RSImFTWhCO60uf/zymZuYwNbuIrY1VbC29it6wh5m9J7Bn7wHVfK1dPS+NOzs3g1aTMHMH+cqsauTps2ysr6K5sy56mBrv8Yhp+kh/8ts/4H3QbCFUye8Hh9mC+lGAYyfDKhRLeeMcnbgzVP438F1CjwJivGVlnE1l8pSo97ZMgxPuGPqo9CYzgeqJN2qhGVq0CBgM+qpDI6mOtCjmzDfW1zA7M6NDaKKihF2XVP/k7TEMJCGyV1S8ywklXYgPTRvLF0/lLZQKKGSyuPGGG/Du9/4LhXWdTl0EfkPlGBV0lQ3kiwwcqnU+Kz1fmbp0GitLlzC7Z49OGZC6L2Rx9cJFXHPtdVheXkKqR422g6Tfwb6jp2RCWFBRLtuYTY0n+MKDn8P0zCIq07No19ewdO6ryoQdPH6bPPJOc0sHwHaHwPTstNLK/V4TufIMZmfmNa619avi3ak8macPq8Chi9SHf+dHRottIZf3J1HHwziT2k5mGLEhBe0ZnCreGp0kPyhUjEo/RMXAA5oDU+8Ww6Z1noaYrN7OcgSqDFNo5efQyS+g2W6g120pxqYd7zQaaDV3pKZ6ZL2y1kq4vbVfZm7aTtyzXR4ghQANP6ScEOTMzDTWV1clnG99y73Yu3efaYheG7fd9WbVk3OxL1+8LEHrdpog/6xcrSppEW1G5Cc455sTWd/awMziohaRqrY6VcXls2ex//BhrKxela/BoorlC6+iunAIczPzYHRSqfD4KFPj1C5c7AOHjomHT01QX19Gq0Ou+M2YmZ7FkjgCqyhVyRGfx/bGhnh9E9N7MDU5q8UmgsYTkzkHC3v3iU7FRj+pD3/oRxPtwniZiR21QTYQwc/zEp4ah5fa7uBLB6V6laPgVe+sFDndKGS3YwYtAxSokmBFaQ1ChoYuDZmTTU1iY7OJrfqmKE47m+tsrYB2py6An+8jt9zgyzTyaibIrhAFUW/Z8oKeN5242s46zp05o5OD5YB5XzPrMgS0egNcunwF/+67vwf33PMmdfl/5pmnMTc9qaggSn051kbdNAjPqpYvkIJUJ/GAyWpVOALHUSpTnW5gbnYaV5eXsdNo4Prrr7fvazu4/ba7jSY9wR7ljAKsCPHBBx/EqVM3YG1tXdy+2uaqophD192qg1fPnXkG2QSY2seESB61zW3UN1cxtecgZqbnVQ1y9fIl60RZLBnbKE50+JPf/qEkCgREY/VWjdEPk7syXsJ5/Sxt6/tlQqKe2+y0pNaNFAw/US96aXpvci66drtfUI4Z0SQ/F5rHJUl4vM3ygWtuxeKho3j2madw4eISVq5exZXlS3Lc1Bd1dhYnr70OxWwa1UpJMXJc3zh4ea8qoZcgN13OA3ciNYQa1w/TaPUH+PgnPoFbbrkD//7934/6zjr+/u8/gce+8iVzbPw4BjmTxKjzBfHv6E2fOHlCLBoVEKiYzzooMKTiTQnt8kU0jZWdWyR4qClRWTa7Up2wolB30D73uc/h5MnrsHR5SVU4w14T/e4A+07cjG69jo218/IbZvYfFBeP8DFbWk/M7cXePQews7OB2tam5fRlwzkHnpn72z/8aanxAOwjTKKaVk9MERVYrWidjvRSQsEWNGykcrFjjdnMsTPnbVxpWBtn7zzgxxf1ujxxqCTkSCfg+HX3n7wVB/YfRKu2jVy5irnFPejq8BlDuRhFMDR76cmnlOyQifAyXFtb4/AG6udDdxKenxDkDNLBMAfCive9412oba7ghWeexSuvvjRKDgk1pBZKLEMXzeLJsKEfEXRg3mNyakr2mKElNYyYs/W6wkzGv9RGrVYPr3vDG9SEiLmJhKnWYYJHHn3UBHYwRLtZUyODZquDI8euxfLlC+g2a3JoF/fvw8b6ppVZnz+Lyfm9mJmdx9raFW2GcnXaDnuX752oKDD18T/9Oc96xaLEQRu2IHTVY+G4+GKMyMZ46exoMQ0UiMW1isZd+dC1YrZdnYcNZ77ZeG86ZXOUATp43e2YmZlDu76NVg+45uRJk3T2YvF66VaziacfeUSTZbVc5L7HgY8mbAGt8jMqDBiZJdvsSln2SKIs4u4336MzPK5cvIiVlSVD8lhPXSAtyzo5jkwQixG8S6OlVXkd4tI0N9ZhgYJAweDPtPkkVcq5K07ge97/flxz5JhCKAI/HOcjX3kEO7UaSjyLs93E1GRF9fB0tLrNBiaKOVXDTs/PY3V1HYcPH8aV82dQnl4Qf2Dl6iWU8gVx0phfiDPAei0u9of/s+9sSyJwN5jjZd0LvARaDlks+rhaJy4rmk5sei/U293NVNbet2t0wIqfejvWEE622lmgUTZz9NQd4kqz9HRzcxu33nan6EN9LwgkiEsy4PNPPAHjjscZnS6oLm3xe9M+u2duywt2fjzbhPLnm+5+HTavXMH66gq2ttcFCAlhcx5ZtJuyyfImc+54RuPa2OWMAthjbhxyVeTC1hq9Pk6dvg33ft3XabcGBflXf/VXsb25hTvvuh0zs9PSIoRl2W2KHZwD++dYGT9rnaghU8DUzDQ2NjbF0WPju+iwVC6woH8LqU/+5S9rZ4fKDRUbReheyTc6fZ04ehh9U6XehMa98dHnojmNfm9N9ETrkZ0mxkwN63XVbvt1cLiK3kzLnLjpbhRLRXD38nD1O+96I5JhV8QH+ges/OA1n+VikxDo6dlx8zFuRsxRsVMLOOlW62VsWXK3KLQ33nU31i9dxubGGhrNbSUQQiEpDeu9xSJEDWaqJYeM/x5HJGqR3dkN4CoqRukLTc0v4r63fb2gz26jJkH8h099SpwAopTtVlPPvr29uUtXJmihA+ZSgqzvu+8+1Ld3UCiXlG2k+aht76hogI6q2Dre/Sn16b/6oGlXV8dsnRFVhoq7YWCFuFGOhu2abtsZHCQJDeEcGcgSoIqlEE2VxiEzpt9JXrTT4Omhs5uQdxvy9OO1N98tpIxNbzc2d3DrbXcDSR+dtpEWCMgQwHjpxedEpzWYNHaupSo5vjixwMa/Cxrp++iE3DcTdPr1r8fy+fOqH6cTx6DTHDM7mUDM20gWceGdzCAz5R0gomOSiIuuScRC8ffaGEijmcBb3v4eVXU0t9Z03ccefxy1Rt2Yq85eVX23OkuRjGnnoZHvTu4AfQGdlUrT0TUYuNu2UwtOnDgpp3Bxcd5qyD71l7+h0Mt2HA8xsSZpRKFMPXtxwKhPib1P6tDroQlUkJkSXXCDdWEPz2YzfmqdN3qLUMwOHkvbGWx8qQGvgTH8/ckb7/TzNbjYNdxy613I8HRf2h9fbGLNr778guwcXxEh0GdQBYvzxU2VjqnwMSxAdeCevrrlDW/A0pkzKmC0fqm77bkoKrTB6tbsr3EUTjZ9LFctyFjQoh3hZEJj41AkkCvjbe94L7r1DWytXpEwPPfC83aWp1pVG8AVTXEZbYRGMg1h1SnBqOUCc/HJ3AmyhX5uNc0p/cSf/1qiRQ1P2rsKEQZUJkdlMFbgZ573bvM3O/PKbqgDUehgSQ17LjgcNnfOwlFidkgagR2FoxhdYZA5TKQv8+up03eKSUpEbWNzE7fe8Tqp0XZzZ+R4MYw69+orst100kYayk/dNQKGTdiIheI2llpD75fmsTHfcMeduHzuDJo7NU0QkS2xXvzc6+C0x7OEBov7aq60820xdGBtHGrLa7Cu24PP3jCNe97xbgyaTWxcPa/fsuecAVCR0DGuqti23lvNSpssK2lA0mudYwaaIm26r0HsXJnLB//+vxso6lAmOwT7Jhsttv4uAiJ3+lj7Z1eJRtAzMMVjldFiCK/2npzhrTOjxsEqc+axLwWHfULMKzfu+nU33+HYb1uY8Onb7lSIxpZdro+lwi6cPydIlU6aqVNbHMX10VB+jEQYioQecoSOAfjceNedWDpzFvWdHfMxvADBivt3SUu249wshB13tW6pYkvnkshh2IVrQ/YRVTjIurIEb/7692ix15bPSdjOnLHjLWNnhjDp7G3vrhRahfehWuecGF/d2EVc7DA7ETnIdHzm47+XMDgfSv34PyfmaZF0UhzPf/RmMxa4CfHSronuAj6ZvImdOGelqqPJVAdfO+A1doEWX9CrxMkaqovsZ6f63va6N2Nnh2yMLlbX1rD/4GEcPHgE7caO4mpRfns9XL50CVubm+Kgx3LwOgQ4RlI/5liJTOiHoclPdDVObXP9LTdj+dJlMWnIXo0+M+HHBIEhTvIbuWxxGq6r6NGCeZM+Cz0t2WSwM88USeMt73gPeu021pfOCjc4f+6MLbZ7/+FjKKtHAfFW3LbBDGJVqYo2kB9O5+FmNCaK45hTn/rb31EMUSyzH7j5nYb5+jmY0TpSYZLtCd5InQ7Ey7JSHCMKGL2YixkQbOw07QS/VrAzQ3p1Yg6rJxw2NcnN4vSdr8fm5roQI+5sxuF33/1GtOm5wjQQr7G8dEU7W2fZOu891DMfSrsjcHkXKIVSLqD8W4BJR05cg621DaytXFFPEiFRHFsY9TFnVnVZrloDHYxdZ6cGBbRsjeN3Y347S6SHDO5953vEe1+7fEaLfe7Mq4rVJf5+T/lI1ppAOL11d6TZMc0YZA3RrLxvfKzVa6KRz/7D7wsuDXqNUYqNVmyOWCBj9tCjzkTqG8qdGylOs7k6scZzmrb7DR5VViv8Al8AMUIlheYV6+jBqCbVzn4TVtdW1FNlbXUV3d4Q97zlbei22KbROvJz0VZXVnHl8mVRbCOc0iLpQBpXoe4oUXeF+jaBsNEJ8k2l0Wy38cd/9Ee4++7bsY+JDR8bif969miU4/6KnWoQjFwzcdG3xZJAMbN+JFMQHYnLI4Ove8f7MOh2sXLpqxLKC+fOGiHSVf04UBU5i5G/4AUOfA+F3tg2u5z34BGYtkwj9bl//OPXhF6jvp8uwRZnGjFg1NGXUpqN8yzNSVMxgSNmYZ/ouQZyZuc8ewStE+fNhpla2z1wLVpPJEkGt73uDeKNE3VaW1tDu9XHvfe9HT0S6nqsDrHFXt/YwJWLl1R/TafFMl9GJjTeuFdwqurFgJAwLyNAiAxTb8BnThaBlK44dYahu332tG8cZ2k70M/T8uOVAjnUCX0yJxae2nvjUBrqoQze+Pb3Ydjt4erFl2VzL104PypTskNndzsvhUmKbBvVeFCYAwCIsNds9Wtp0akHPv3HCZvEcbEikRF2wj5odjeAjlGHP8XGpto5SOFkyrCYBiDqFUcbSfKVMTMzoZN6vM5bu+s1xQnWYJZlwjfedieuXFkSAZF9vtge+g1vfosQNMba8fCbW1u4dO78qLOhjd+gzXhZZskmWlThcC69gI4cPOLyjCgsRy0RN36dkn3m8UYyJeLqEOZY9N1FlTfgHrlpDyvCsMZ4pC7TQXvj13Nn97B66ava0ctXlrxvmrFr4npxX9G8YiMyeRKaw9GeCNMsNIOyfqbKE6Q+88n/mZi63T2OgWzQkPgIAeiI6Wxt503HJNruND0tD9CPNLJF9ERJADY6dshaPlscGWrcvGe1+VANOFROdN0Nt+DKlcsiGjJe5K3uuvtNKp9ts10jGZnDIXY2t7C0tKTF3t0NnJTdHSV17tWRHKfxvmynh1Dy93TqZA+9twq/l9fL8NLHGyf0CGuIvqD+jCYg9j9UXYAsdhSym0hWtaQzeP1b3y2zd/XCS3LKrl694nQwW2gzpbsHxIiE4EWAHOO42tZ9RjlFrzVztFBj/cw//BFnWotkDEmLcUOiaHPU6DVtao7F+uqsMmYDxxeetczRRYg2kLHsru0O6lOoNNMXcRC7YlI/gJ1O2613vh6XLp5XcbmOccxkcdfdb7Z+afXaCPAgAHLxwsXRafajSXK0xjQNPK7AAAAgAElEQVSvh0puasxb9zg7doUgVMMR5Pw4SCP8OfBvPytr5MCS+KB22t5wncczSSgClTQCR+z8kXBwsQG84b73Soiunrf4+tKli6MTl0zQrKCB9xcnnKiemxRGH6G2Y6FDsEJj8hoSCP578B8/nNhxjP7gzh6hNx8XEgDiKpHzF2dHMakfGoEDVmd890AD4YrEF+fT4j+2prSzSEjmkzepigqj5cSk5PMl3HT6Nly8eAbNWl0IGXfg9TfdgcpkVa24wtPk37mzFYo4C3bX8x1pcn0TDiHVdnw+nMj4uxweXyA70NVACk+YasxU9zIjDIc8XtdZ2wolY0fSNHT8aAr7tKAdJX2ETeL1971P110+94IW++LF82aHw79RGOzZRvWIsYPkLTHz2ub7Sj2PHEKzmnHagFDSz//TR/ycdPPiVJ3IAckxsA5CmhTufH719GE81CiTNLbIeix3vJi14e6WpvAMWZgIo0BZmYyFDLsxOG32DTedxoWLBDi27RhmAi8Ts7jpphuxvbkyMjU8Punc2bPujVvYGBy0sFcGUY6Lnjkv2oVj7SflTwgxtL9FoY5Br6aZI4YOkmOobd4rMoYyYd7VP7xyhXBuhzWSYYJjN9yJ+YUFLJ99XkJx6dIFT8zsEkkS1xaMDKKq1Ha9JX9Cc4+bFX3v8xtRTurBf/qI5mA8WcBBy5UXROdsEpEIqZbd4Pvp8qPdYS6It0o2BIfgCr/GGV0kPASiEzF2TJCpmzghwHb88eMnFFY98MBnMD8zrf7m7V4a3/QvvxU7G1clkRScdqOJJ554VIsklE/OmSNebqujowHllTnvXZ/EBCBsXxAwKBzWsM6OUQqKFT+vfi2+ix3NlyCrSCKQNkcIzY8wGrOcRO+faioshfmD1+DosWuwfJYdKmpYY6gpLWKJFUszO1FEWDjPzbYiC/V1k7Aa0STmdmS7vcFQYA2pLz34vxJzauyhTUpt0qRu2GBdyQlzZlQ3xPeN8dQIpqhk1h0fE9rd3t4SHnVGcI/WVVnYwlDdcX/aTd6/1ezgwsWLytpkSK0Z9lBvDfHP3vcvtLPpuHCR2IjvySfI8DAVqSOYvSWnhMpNk7xgn6jY/fKmvdWlhWzWuzvUfbBrHdUd/T52EcMqdV3gSSd8U2g+PxMkujSquTZbcuq4rOixDmTKU7iLIea5M1psljqNvH47RNPGz8+Lym3FDPaKGF5++2ixw2FmOXAwSCTsX37of8lmW7Yodl4U5zP+cFBE9un/a+vanuuurvM+siXLsrk4zTMdGAghJc0Y22BjoLSZ5rl56kuf+tfkodP/oy+ZydBppkmAkkkoNrbBKdB2aOMB27JsS7Isy/iiy+l8t73XUdEM2JaOfpe9117Xb31LXYzxtLvTwR4pSR9LgEZeVpvIk5QJtIYnSxJVoAiPCgRAGTpVePBnQizc79H2pJ1+/e32zb11xtpsf3n8qF358ss+WSdIVpLteGFyvWrBs9Gx1QzLEJWYoCejJ1QnF0gDa19LpQHqjKhFJoxQa288TyHYI0pGTcI0abtzi+3Ea6+3m1f+pz14uNlu375pG68hOVhPcdqonJo1wXvt0kGTyQ1zlMRifHEtAgP/+MN3kgrhZuGHkB580V4nVu2D1nSxWD8qy8zI1O53tZh/opU2C0nPO2AFfxbJfKjG/Sc8JkA8prHvc+2Vk2dZDHn0OM342+3alSs97MgIKJ7ylAvLCU6uoJuqMgVQalnjmkZYpU2W5jGO3oyI1GY9RamedAnPKBgBlgQAYrQBrquDMNd2JofaqTNvtLWrVwiWYHrYqNVoGBZhzHmukM5OngfohMUh19f+qCAUT57ZynO/+wWRKnFociFCiJ3qRFYLtyAQwOq8k7LtG8fESlBX4QYt2u6nt5kSywXWwpBxCKrTIAeeOEnQjG1VgmeunX7zr1gQQC8TrgPM981ry4ImdfuVCYBKZgw5hC0WsIGLY3oLLbBKrqlmqZ/NiFW/p+RTAh5SWaP6ugaqmwpsu/7tqlfSpTxYmKh+qJ149S0WQkDTvbGx3hEv40gNkASzcp6AoEepYazVuvMe3XYnawc1HrTJCFdU4406pdfZbbRjYdNAUkpt63Pao0T4kvbMueIGFqpBXYstG2SmJicpFFZgrPAAMOq99FyvvfmXpKcAVQe5UnYet6t/RNVoh/9WGFeRMlrsLB7Xx+YJz8AowA9dVTun7iH37Rx6pgNFjQOmS7gV/BHWA3TiVD8Y3j7u1zeIc7vAMgVth3U92E6++jaZHzfvrfNkax9k4uJYZk1xVX6vqGrlPGBf5LDFXPR7JtV7/sN/0TmK+q07ZueAC+1eLv1dthsnAMNJ1K9tUJ5TlXJsaj6nPJ3Zi4C9Vi+YHERsR8hnnLB3rK/TFOfxe6Cu/s53ScRD4va97bb89dV27x7w5KMql7q2RiaBv7Q8g/8aAVdoOODFiU6kqFyT90LSJynwJPoeJUfOjeiD2uwxO2Wp0Y3yReDRo8x55s2ftDsr19rdzVX2d3HsYuaTs4xc0rV9/Sv2L1UwPKfEQLG6BtoEmzf5+KNfWhvY1ibD5FOZE231L3XI/8+Rfjqgh8R0OhlyukAGD3uM6TScqxVbvSdmhJKnV8HERQeGPSyJJvGhaBfCxbz1wlI7eeo1MiHTmWq7beXqdQLzMk1eWkm7O4odKXJhBomotjnAVKatV+jkUIVpSAyPFMbAjqzNkkJNbE2CeY+TyGQAMjoZuqy5W/DEVeAgwufAQjvz5l+3zdvLbXVtpd0Bu7OdUzw7ng8jq6kNSvGoh4LVfyrIWWpVb3YO8uTiuV8RSox4MN7zrPxLavIL6c5E7hoLMsKA2d9KzMffcy4XQkfaSrSpGqCYe8bOzXrII3VL5KYF6e79x+3tH/+EuC1K8nSPNB5Qgdg2fTYmQCpdXrQ96V6lEkVHHDloCWgBYMz43LGHnPGl9ClOTNS3snWKh5FnZ77dzh7Sy2Ql3tPAG8wCwbVFSARPQA4UNvPlk2fb1vptjuVYX7vFe0k51CaMsgeZQNBDMK19F+p9Cgx97TzhF8//2o19Q8fFfZcS1qnqm20Ok3SI7BcQCcDYJHrDO2itfaiGOzaGuz2ocJbgaSAAsy+pxj1+z2kSXH9j61F78y9+3DZuL8s32ttt6+vrbR1jLayZ9LzJHThvwFh40Fv2iCK8KHZ8sAEsBvnm2EBQhuTa+X719mkryc6gUcbpfcv6wCuI40n8gEGIWOOXT73RtlZvtdXby+3uxpr6203Bid8H71miADwLINQcBxFHLQ0Y2WQntKANuHbOo0w+Pvcr48a1oYq2ZSP6ifZb4nvzC0JW5gTq1CTcGDavxsg4DVBlcsaCWvUm2rusmiD935BUeLOS2O5Cte2duXbi1TNtA6dgD1TVjQD61bVbXaYZYbg2YQnqJ7UKKN5JVJcgBhCsadaxlKgpdBTIQYKZcq4SStKOEh/6AbbjIBzQ9TAZQAT5aYHSlaft+6+cbvfvrLW1G1fbPYApe11cCS4Wh+y0Yj16+jNxvN86BzJ/ZjGgzum/fPrJ+/TGe87XKiRqNb8QFYV226ouqtrdpz1mBCI2T+p1oCFHBDAECCafaUerUiRzmFjh3E7QcB1qr5w63TbXV0lnhc1GVeyOwxY9B3qzTBvhWLg/X46odsZwXyWElFoc5EGs1ZcCDXVdSrbOlxPznjCOZV4lQsgOYZydfADhzxi5USUJRPjD195o32zcabevf9XubK5zs3ELMkfVAbR+NojIE08cJeKOJU+/x7etP01BiAAvXvgNN5ujkKIyi0cH0Bq+hG5UjRpf8H2wAbFR+3PN/Ey3s2Mel2J6PVbCL17fTkw2qsezOiszNeLJ3lw7ceYNOmRomwEVFurda+urM2FXMnYUqHjLAe7vW5nkxvPtekq0L9Ze7DEDoTxoLsBtLt61aB8mobxW1G5GfDLxEu44ok1R25cX/4MfneD1bl77st0hnQgcOCFMD3pONvYmpLYH5kWwHy2SZ0a/WOJ/ijsPixIstNkXzv96mrSe0p0eG8GN1WXYQOAZzIEWIc/dL+i71RM/CgujlDjgsb6uM3bJPwe5mQpVct2Kaw2AJHFKa6+cPkuqRoyMPAjH78GDtrJyvTtMqqPbZsXw+zlzOpMAyp8Jl7KIPZal0+I0qHMC1BzklgFJkNPNwIQDaMdcuzppoImY2vSJls4ZAEccoOdefJk+wvWv/ov1akQ2nLyEWjbsL4afu0NEiS3BrWhanOaWMI5iiEJJ5eO7N/7Jxfd6R8jMD913NfqmZgvwcLoYI6ePiDnzCnbDyRWqcn96tGqB5Md1kmvHpU5zCHPTXMeOyvmF9uLLJ4hU2drc4MlGFm7l5o2OF0tdW0I3SADY2xVOb6NjcjK6SQkg0smLaAVqtzQxWoDU8eFChVU5N3TG+ZTDJg2pJoqOI2tz7cixYxza9tX//ne7ufw1JxbSbNmHSpIIDpmG2TSSDsATUIg6Uqj0j+LQGrZMDBCe8dNL70+hluSAqBdbR9Y+kRMgWNioA0gKOwVdyYEdQsNfWlajgns4ZUjTQFoWtegFzKbIRimRoahN4Q2+xEwoTTO/+FT7/kvfaxvra+yUQBsQ+LWHRrFtdMIoaVTxgkeQMJoYU4+GY1nbd6qmx6IKqKiig/B64z26AHf1OTQaPoj2KHGrylZn+Pt0Z9ouf/FF+5uf/rTduHalXfz9b9t3jj3J+QfJjDG9y5aoxmgGIEgWeTxsjvjBRDhss7b/Yx9BDt+0Tf5w+QPS1ygLlLgl+12a9N0JghoqnAJwimUze2xpG8GUnoefiUZaeCxtYkIi60Z6uqlj25O1vOm6Dv8ywdaFvftb2+21s2fb2q3raqnZ2WnLN67xwYW8CdiwJhZ1/yAyldQaoEQKMdWkCzelb6tv/AgKVE0y5EfCaEfSCy7BVP9XNXFxqOqTra7ebh988G/t5PGX2xLYEiDkOLEGIdAEGlARcGgQrorHkdUDH5oig9Tgtd6mOMPJ5oPkQlalLKCzJQeDxlE8iJ2NLRinI7ZbiyeV5nRy/xMbqhYVLXYqO/SwS3IAzxLkClUZF1D57uScITo725N2/NSr7fbNa4T34HpQ4xAOaJioZIQq1AxpKS7v5yBToQz5VTCkVJuTtJqyqCqQpA5dHUuxUth/KSldLHFKwqoejnC2JksYpcB32d0207JnDXAtlQxi+AZ1jfEW2zucQwZoFt6LnSPBCYDwxxXL6lDOL5joCKFXjZmT1sTi4SEB36WtsXTizxj8bEZ+P6FSTz06hNCNh6qUDRd0SDEkXtQUlS6Q8HeceZMwZdYXBEA/Ovn6W+3m8lVgSLlRt26taHE8CObbMoI5BTFVaEmqz68WWzk2KnP63YkBB4/aYqfPBOYMX0ySlNJjDVsxIE8lysIeGJw8b6TcNZJO0n6D37xGBLTNHALPxXArspklQDO2s0NOuHtb95iKZqOCexnhXzFE+8OnH/Bk9w2HNDlbJVumJvpsthIk+jyrRQnF0ozmPHPQL0mpjkoQZosM1TnrIOhfeDC8PPovgi6hSvToIjiNsIEnz7xF/jEAnHEfqPEsdGL5qPP4EdFYET5ojapOa7go10WFGt6fm6PWpkQuNDJOzECFIudO79ydKGSz8xcFLSFpcQiUANq24zjajqMxs+manKCnjXCR/RkEufb6EYKCkpSQMnKrqYjDeWXZbJbnAhEuD8JeLmdw6oZn07PxgiHLaWHzuGdcRp0GKEBuEoP60BbcwwID6HU9WbugJ9FZwhAE6plqEz+bbz9CL9gaxkI+pucKB024OYdp6QFmbV5NinjAePhpeNMzJKmihnvNDpFGUZSQaESCykDHTfrcLJxId7pogfU93Pewiz5xDHNAcmDI6eJ5nMPZt0BZ02WdsjXSXhJysTS5X85FFDhyqk62Ptpicuniu+JUsXwn5qZnTika5bO8XCQuajwbSu1g+yhbaT0SRKUXVQkUdW0yBjX0iPAbniAFD5wGCRI3jIYKRNdcIWgP+sGfnyAPORiI8LV8Q0R1GuCq6hKEjjPLYJON6aID4znaCZ34bwq7bDcWcjbRkky6kiEJtxiuWhBjfxlaudFR3Z9qicY6UXNgpMbhxe608eCkJ67jzmd5YeL8cfMOmDQXc1p69+hen9pbBQN/R6jKwfCXPv5N3qKoKpXWuHnGnOUEx7mQsyUvOw5RVB3SfLAb8sQ1mTYmS6xC4u5OD1QnZvP1gv4Erhz8pVWNcnQkVOP0QHvm+Re4qWBTwtfNWyukn6A3ySxWAAvyVtP7VHFawZlhpHIydTpxo5iT5E5MQ9VG4CvXe48qm0yiT5WRPemw7KwUtuOBQDEK4LFOAqn4OEVtx9xWf6mPniZ0GcIoAYxGpq2HULDEabWU2LFWpTicmV8KnZhata2m09BbXUZlDJ/FaKI0ApL7k4wOJTwxL3naUxcwjQf5ZJ9u3BEErBpBLCRIQiqGRm2+PfEn323PPvccqSTxhRInrscMAMD729tkG8LG0dPmu3gRDaiP/dVwtREbd3SttRP+LSEbBQ8+OzabuYKR/lVUEpNh6k5DruCvJFNY07Cxw0Go5ARjU+P9x//JhufgAcwoBy5Jd534oZm0T5MLH/0rq1483oVdIBs/c+xl2fqm8WYHNMwktQWcZHCNcpSEpYs5Yo5zkMqW4GhhUapDe5EqOQbtO5QJCyEhSsjWOXTDS2AMIRrjTp89S55OfA+c33BQOILJbI1KWcqRxL2hbSKgSiIp0zcSOXIKs8AAEEbFwjT1EK33sMthGrWV8W69JOq05nAexeeuTXOiaF9KF9eMNoWwc/18GPJs+TlOblXz6XaJj9A10acX3p0KYTEQFUmu0AmxPY8nrGFPQwTojZY4mZOBZtKecnIY6/qUZL7IiKPtnTvMgfCgiiU7rWIB1ZDVssp9ILcDWO9UW13RlN6Nu6tkEEJ2j+zDYPhzxSxISy2iMk4anrrN7s2kN9PrhQWiEBotk/KmzMFgYooDV52umLeo/ZiebDYrab16WMD9xdPucbK/V0NevAM2P/kJYO/w/ELhylzVCCsagDabF+bpHl2JSONFv4v1aFRRdDId4xkpCjyV0psD6Ie/0zFQykhT64o9g4MWPDeegW4ZhrK5vpzSphZ+FDUEPFTv2Cuvnmkr167y5e5uronczYkdqjE3K8ZZVNyMcBJOHGrSek+ke/GFgkpMC+7BU4TnOuAikWktYeOl9r35hjhp2BycOxs/x+3MetnJ1MFBfludKTBP7Et3eKf9MG0XES0DRcRN5vQDHM5RtIr2JC22U8JB4cSBnpz78JeKswtTLz3yvZEZktrTw0hy8AAOLQy3ibSl8Wx42cp88TTCMwTkx4uEFRmqBpkSXR+4NQmF79VhROJbSYQA7rXjp063G1e/5qJt3d8gYgVCxdKsNUV6oiPhym0btEBEKhZdqBipSxHQJ2rgOAr3VGX+p5Aoo3Ajpw68brovpBFrgPdmehmzxgszFKpcMS34LBNYKSfjul1/SqBSWuY77Gl2N67fSXNc3NFUxZiWcXhpsy9+/B6LnWH94xksqqOnMp33jqOGFB4+BqaeWdugGVgKbVBnvt+WOO9aJzfM/iwPTveYhMClU8+G972I4kSHEkNbiJlQEjq0x/bOtJ0+c7bdurHMzQH98vr6Gm12TwyRqQnZJRHEQjUne8dqUkh7Jgca5lknjGKumc6oHDe0KjOGR1vSA00TTn93PO+0HkOYMVtLGyikqPyA0e0Slatr6oTCvMmpVVwvhKlgVPiKiYRgwy/Suks4a7TUEy5WL9xoCEnd7NjQ/FCGXW4lZAWSGbUGT5eDUuz49MDeN8DpTBtwVEzKopmDOUhwR4GCqp+w370+sD2AgIAIEepx8+cW2osv/Vm7uyZ2QHCRX7++zDHInNG5s026aPGaisRWeX45atgcYsvIqCBHM0PQsanyDVwx8nShhGVDaOVgIfqginU+H825+uwBhoP4PLBkAQlkrSEQ2fCUhKN2c/BynWQy8X1om5rBjOfdVbYrez22Z+jFk63TkpvGkajA9rSuYlIffh7JlIqEIKiYEs8RN+8xcWcDVp4Ym4CXxwMDyYm5GrhGkitwsLiAbmLTiXHNuKMolZR55pnnid7cxcjG7Yft9q1bYmBIWLgLFWlqjU5eo9HJQXsQLmQikRAJcBNcIOEkQA+HBSgCwgh4b4bajd5ybW6yWlgLCCiETHkJYMWlIdI8iaQLGvmjqnFtrgNO9UzBTodOZkbTCuTfKIGEZ4BpwM+zrvHQuwBks2OL8+ewJw6H7IFCF3Ni3WGoZn2JamR4h5HIJF6wcHHgEo7lMwT68T/E0wovSKVpcLwkVlkraJP8nDXi6bQdXnq6PX3saRK9ovEdDhoHssGjNEpDmkWxKE6HpuSJ7opwXla0RPADqUtrUJxJOnT22IMQSVO9FlKsSAk3Ewfn5NHj3xZB3UxBCNqyF5ZS6gUEWQPl2CJtxAvuo9hfMXRYDpPLx/tRU1mYoE0gBKHepM934fy7PY5KPJYTJifdRZJCCSkPO2KnP6v6CF1HBCcaItAibeDwvOvvihpT6UyoRhVCNB4i92WSBO2rjx+3g4eOtGf/9Fm2Au3ubLfVdbQEyfFDEoV14eku2RHiiCoxInADrquKuatXCBMJbHQPd6g4IVydiK5kt6zm5YXvtsXDmlVK/8CtuVgH2VRdm3l+1w5U+VPuQRnFsZZsP8JweAsl1gyjkbG+bFAwVGvUuZXNSddJNDQTM0hqZbOTcYlKr3ajH+GGmRaa5BrpRYkwdk1ORkhsArcdUJ44cvlcEgVJFQZUgJ9jQznv2qMaBpOCFTrGP8LxObjQXnjuhba6uiLmgqt/5IJT4OLFp5l9H/BwRssYANE99vCrOvkD3nD9TJtBzWGzpbDQwm+kT0LKqNfkGhA2xbGSI6vWXmUItykETASlrm6wJwWyx+HGFITN2Y2QMHS91h60ivMkPGBffPbvU0gWbqzyn9R0Xjqbig2A5xwg/0gc2GlzrjdqpSaEEuPGS8y196dgByugVGPgSLGjSSRQLbtmjVLn8eMnCDaEqn3n5//UfvjS8/LaCb5YEG2XB7+HmUGU13a+vE9Y8NFtOcq+FE6nP4n/DkOzt5hajuXLAtLs3RwqCPW0rFOyma3dq2k6QqpVu7ukE81mMJo1BIkPWKNSviH7ldw6NWlICwsMmg5aJDXNbPhw3H1me6aN9ihtMREAOQAmijfAQGHUKEAkNSoEptCQ+BPCFQdCp1d4ctko3XMmGgj0Ju01ZleEnf/nd95pZ86cbv/4Dz9rf/93f9sWD8+3xUOLnB8GbxueNuNSsCog/jVlCEMbb3TQKR0IWPq7uA1u8Y0GDL02n7Hi0p0jTZMFO1fpvLoNyZzobAVWQbiXJ5N3p6oHHYjbh2nWDJcCQzPeGeu4uLRkLZsSrBy43vi/73RPLl14b1pZimJ/ZZMVf2MjOLBlH8mNPlP6hVPJ8bG+u3G3PfX0U7LplHrFhUlyKMQTLzgkP6paDs8YDRmTEuHA1VSSVC/1Y87sRBPhw3ZwihLnNz7JiIkftKUlTNgB7xlCL/V7YeKuSAKM9nSbrwo26ekOl5uydez88OmjlvJ7xjbG58m/eZ0219bW1zgkhtqFhRiphK6u4/OUHEc1p3aKmJRK0Yoh3aNHjCggvNG0iumFQuUhKpypk0sX3p9ubm4yoTCcrlrBksUeIL0JHSV41wn6ZcNjmwPzGaBD2ShVYSCRrF512g6hNdNWo8+FL3WEY0m8xF/garFeiGQDxiIjiy3BTCZqfjIhXgsoEKxv4lRQXfPkmesFz/fNN1vMpYcbpfssLKjITmcqQA6CwBpKM6eDJQjcVEa6s1vmqGSjKRRutpDGEeZOTJFpNRoeU54pthtTgZL8GTBuJ19szyM0vBc2OxL57U6ZbiZ77hFNpeEbkqVwJCeieucSfgLj+u8rohWFpuJu5ZI9ycBCoSyXwQ8u0EcYR5Sga89hlBHnj+gLagxOk3LvimnxBRN3//5WO3xoUaB7xPHz8+3QPOLgbaVQd7XoOAAYldSnHIw17/6M1kOFHsKDwEQcjHotItG+ptgj4j/AhHDqMMeD/kkn1TPmb6YWoG5PxuNYN8dPoAUPlmCsDZ5JPDShCoFJo4N2+ZPf9s3GpmdTojKrg5bNrp57PNrYOth2Zc6GdqAtBidocN8Zv5S5GS44xGEj1bJDF9zTfaSdB1Q+geJ7OVomk7U9xKhGxZdqm03SvWYI8bzppWIee6IRj/MW3m67HSaBxTDpzhyO8RwqicYBlUPmvHRYD0ImaEh2h3V11gph/ygwKI6Y3A4nPp8VocCgueRmylPrzA7adIV9cFjjNPJk/8fl302JPCzzr5SEGHTGRajlWboPORs9q/5lnxlzLqonKaceJy1pPZ40Oyg1BOLfozatQUgQU8hsc7+Mn8pmRwPd37rfjhw9qkEpHuGgbNkA62Xj6Yi6GY+x+67CIWwe1b5LuECSJgYGGPLOnY127Nix/2f6IgjQz2n4i9qWdhnVO4aedvwQdiE7FzPFOFzODu8xYGI2qRMBMzmG8cA8w9T8Lip5iXhkFg4wvp98eumDGXxCbHNOeAXwRwhy2hmse2J8atjZCHnYvU6mGZmeZ8Eih73zOEP99+yJ8h7FAcLCQ+UlYpAfIMHqwuZ5liNe1/35Lv4c1X3meblJT8+g08HMFNbYyBPlx3MPwZ8hCIFSJSunRFBoJvX5/VqxC2k89jIlKbZ1HAZBmxSDay112jXgHZ+7t7nJwg5VPFuD9sQV68YFnHx8v5c6ocbjIWsBRzEdL5qXIpDPbSfDSYqNnG2pqfYDf8c1qhbQQBi03oxMnDzYQTyjQHH4CBRyjDGiFtImI5SS1BvAaK4xLBJ6v2BSxvuMal7i+TwTFjNdILDdMDlhJkz7boQ6WMpJKI8AAAdhSURBVHeFTPM9/Rqn7SGm2TLZokWOZ87nJ3wJFTxtWl2TCMY4SHD8nO9wf7g6QhVbU70/gokKBbj8VZk1NxaWfAk1xOXLv5/SPhtaEw6x2G+l8gZTQiQvdrtWYvAgyYpF3UeAcpry0hEYwXoH9kzJj9mxilGfta0X8SbOrainFL5xRkhaVL0IQbf0Re8/l6DqkMlOjAVPn5g1aY+5NQmIGss4M5qJEPO5g0MaT8UTrB9ULNYFEUzleckzVXufE571iTnVeqpfLHYYzI442VwXLazv6VYuv2tMwOSzzz7iZsvDEyYq3mtuPLJiY6pMNjvqvnrrWqJxklIQiGpXCJbWnrGxuSayXimPytFTokYxcwowOfXwgBH/Aq9u4rze751JQGFuHAmfoDxiampdOUmdYQORFxdiFT8TJaZBfGFWNudKjbBy7RD+5tBwhBRNgRJSWQtBqPT90cwY7nIsqPP5ps0A4RBKuHpOTQfsozhKQ2OHlGGz8eHqqWbzUz8epzykqFC5QY1kY7Upo+gxWoaG/R/9xFGvtQ5bncR45ji5meKjk5ci/igYxPGSWgRXqVOdTswM4cvfIoiBGAffpsORcIr3Mxl+/02364hFQdGLBFuqM4DGrBlMFd5V5rACE3WvmkmMd5/3UM1cdfZ68GifbVblAMuRC0NEogL+jgs+9Ds+//xc51SpH0p5MKiObE6kKDndqp5rPbyq8bHE+lskOLadoUahg8qmj2sPxCfGIIhZUClQePxaCBPjwvbbYQmNNq6TGrJSkE7d+lQmWRLnbzhW0tUiBxi5+pz4qn6x2XHWlMMPBNgJmd4TDm4ZIV5qwTo2/969LQpGZ2xy/h73TBkzZgIags7XnCpd1T/oG02NZ8QrNjtSk1NWN50pOvdJMzXKAWUhtk0hAY1pGBAumqmqKbJww2kbZdMqEJHq2PiYAZkQJVeGV6xTgRQu0SX2/BGC4GVUsx5hTH+GjGvEe6BZgfPHFCb2cMvJnzwP/qQ69vgFePO5djZoqOtBWJDTCUEJiie16W9zziJAua+c2j2GeEAE6T2Vas7BgBMatNDsgTKYz45sYvfJF1+cFw9anddRSlYjoaHm+AhGbJaVeMc/V6ejhh9V6rT4aQ0a6jhCNpw6lDrdb+wifjYuzxsBVSZPSQdWoAwqYJxpZ4mkcalU5cSYKuvBw4fUEuRutIOVEI4LzchE+Paoea/GjI8Th2q/TzLUveJkkcQP9RxBzmZn8/P9CBQg1keOLLloFKbkUaHTvjjTZh5Xric88//8XDZbLrw+GDWkgsUgcmNhxMWOvExV9yqciAqK0GSX2YT+UP6bed2OIEHixm1GrhvHo8c1hkerNtZasKnhHTZDi2xwIBGv0DI6BQinDh9eGsCA7n8Hj65wCM+IpEo2O2iQnETew5oDahYLOBoAM21wIGarxqwaLhmxmouoMbjWAKp+ND5mPaJpIgSgBHvyyaOMtSHJ/YAZCxw7zh1WnA0vT433mT2ZBIqw0XoBVprc+hNtkOZb/Vt56H5Dj3msKoZ22JmsEepI3qr5iGceCR8/F2xoVqWbu6yGHkUooRJRi0fOLoBJBR8WPlflWBErPK54huQa8g7yA8yYmNGI1hJxxMhs6CRLTqScqoH/jg+E90h0UgWY4bCLRtV5zufzp1S6+VFNeAAPPbTfSSbxmZFBq55xJEc4LcGH5GVrI0EAQ8fEpzbSmbId1zDcV2bQtVfWwQL5d+gngCiJk7V/w7UnmQ44xk50zeLwUvH0MDNYhEMkiEOodJA0mouHl8hJokze6GGTf+DZIrPGr2cBq9kQkFBCzejezmWEPJue39H1k6cfEYUEwKEVhxBopHUEJEIg1a4GSp1wMSly0KyjBX7fh4BTfQEgdXMh9hICMJMujWRp4VVPjuufF+nqPjXYzgIgz5WntcTY+G74TmP0qTWcqWMt24akdk7GpkvCR9twTnwWJPY/mw2nJeqf82bNTMgcOMuhYBnU6GcszsEF0UzVzc6192ukaBeZORMRWJtFSCMEw2fQy+XfEhTXsn0N2nN7/DtZF/8shy+Ck/tqr9CSrGIINS8STNCsPjwo+vJQhEwAanxspLzrYMJif+Nc4PuCz6rmTKkMrpr5ZJUsuTlWCTOJd6vW1H5xX5QZM1YqKjtOVcITLeAgxgkvSxy54cmbiNbsDTwnlPgQ9nlSoPlX8axy2NCgGF6xkf2iBpvF8/YTHRUPXtCcQDx3nLrYeTbulRFMSHAwDGQXrUqwOKXEoO3stKWjRzsQQSHfWMH8HUxK7D1zFm/A39y9KenyaGlV3Kmlocbria6OQiS7OkuxPbKD8F71QJ1+0r9E25yGP6u8uvFU/24zDYlrdVjiE6g47+S+a+PDdAxgdU5U7CliWXB2Yqgc4LoLwHujros6d6V4dmGB7feO1SNssPOY5Y2vsXnjpPJeU+H3EhYpATL4YhB/R4j7oeImSVvBK4eNX1wQ5psACg+hjQboPlCiJm72nAbYl0oe7TS+7/73fRjI9n85OQ8T7wFtAwAAAABJRU5ErkJggg=="/>
+        <xdr:cNvPr id="21" name="AutoShape 14" descr="data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAHsAAACkCAYAAAC3r1GFAAAgAElEQVR4Xmy9B5Sl2VUe+t0c6t7KVZ3TdPfM9ISePIqDRhqhZAn8DMu8hXnPmGXAawHCZDDmwUMYk0GABcY2wQSBSBaSQBKDNJpRGk3OQTOdu7q6ctXN8X/r+/bet+7o+fbqVene/z//Ofvs8O1v75P6ylfuTwaDATKZHDKZDIbDIdLpNHK5HJIkQSqVQqFQ0Fe++Du+n7/j116vh1KppM91u11kUmn0ul1ks1lUqlV0Ox19bjAcYjgcAAkwTPi9XYfXKxaLun7cm+/n/XuDvq7fbbfR6/X1Pl4jneZYEiCd1ec5Xv7ni9eIMfIavC7vw1fcg99zrNlMBvVaDYP+ABOVCjqdDiYnJ7G+vo7+cICpqSmUy2Vdj/95bSRpNJoN/Y3XHQx6+prLZFGv11CpVHQvpNN6P+eB9+X99Cz+lXPG8fErr93v9/X+mAP+rt1u6/7xe36en4n38JHHfx4MbL1qtZq+JgO7ZjabQbFYQurRRz+TJACyvtgcDC/A/5zAmKj4ykXW4g046fZ3CklMLNcAyVDvyWSymkDekO/JZCgIPc46uFx68H6fP6JSqaLZbCCTztjkcuFgg09RQAYDDJNE10mlbHIyubx+jjHwPrwff8eJiYnm2PL5/GjSY3K5yFxwjovCx89SkPj+drercU9MTIwm2+YgrbEUikXdo9Np6bq9Dt8/0PizuSz6w+FIiDlPMU6TBKDVauna/Bs/z+cZF8zYWHr+VErvp4A1Gg1sbW3pd5VK2TadhDBBqWRj5TU5tkzKNif/a30eeeSzCW9EqaBUhzRmMiaNsWt5gZAwDoSf4QXGX3wgTjDfpwE2GppkLn08kIQ+AbLSHKYN4sFarbYmm/fkq8MBZzJoN1vo8/tsVg+RzmYwMzOja8YYOAl8qPHdHRPJa8Ru5vslKJkMEkp9xrQDBW44sPFo0pEaCXOz0USn28G+ffuktXRPLnCvp89QSMoTpp14T16f8xC7lb/jz3x/aAj+HEKgsQ+GWshWp439+/ePtGyMnfcZ9Hsab284sE3A3ZskyOZMI+dzuxsxFlnP0uuaUHGxbQdkkMvGg6eQplhwx2ezI9XDwYeKp3qhpPPv8Qq1rxtQLfUHSHH3+04P6YWEwXYIP8Ndwr/x//b2ttTOxEQF2byZEk5Es9mUFOt+aVPNMRG8X71eH/0cE8txUfXHK8yGFjpJkKdK5GK128hkM0hzTLwfhaBQ1L34GalvQIuhuTIjos/SJHXaHZTKBY2fgspdSIEYN4tUrRT8MIn8Wwidmb8U2u0OUukU8oXCyByFidI4+n3kc3kMYLs1TClNCe/ZbpugmrkbjjZNMZ8zIX7mmYcT7hqqU74K+bzZwIxJTbw4UP6ev6OEUgVJsoecexOOUCGyYbk8qKz5no3NdQ2CExFmQjug29X1ymWqnwES3xm0vnpwV/cxCqp1jqPX7vBxkc3nJQSctGq1OhrruI2L3c3J54Rwgig81CBSdy5wOZoPJBgkplI5YVxYCdtwiKYvYJg3PsfOzo7uqUV0/6DdbWsecrmChIjCzvmlLdd8pmyhzBylpJK5cfjM3ADtTlv+QzzDxsbGSHiq5Qn9jf7EuGngfIdW4XxwLkJ1x9+kbb/ylQeSMp0E38X8pe1YU9vhjPHBeSHZJ19sk54JORJUg8WiSbfZNu6+oSai26V6tuuFitNuGZrTw50sByudNtua0KY1sb21je2dHZSKRRw6dAirG+taBNpH2ihKeKjDuG44llxYTmjsjBi33i/NQ7tb0PWnJie1O+kzFMsVrK+tI1/IY35+fuRvxFyMa69mo4Ecn6/T0Rj17IlNfKfTs53X72sjcY6pwQqFnNQ+BWVlZUXjp/ks5vJaAy4kf8c55e/54nzKbGbMNNCMhXaKv8VGDBPKcfLznA9qPdnsxx57KOGH292+VEkpbxKdSnEf8UY2aDpwox3mNjkmOLzyojsLcsiovodDPSQH1u31sLW5qZv2B2aLudgUECrJGKQW39XpoD+UWjOv1zx/Si2FiLuF+jSdzqDb77k3PpQnigGwuGcR9Tq95kk5W/Ja+wOZjjTv7d5uJksHic5kHu1WC8ikJQx93y0lqdTE7pGixkvrs7LJYcYonM0mVldXUCwUtfuSlO14037uZfNGqZTsLn0AzpG0B4Bex7QOhY8CxMXms/Kz1CKT1arMDl+r6+t6Xr4nbDMFM3yEiFBC8MOZTj355BcTqhpkslJFGdDB4ETa0vZ6HQ2aaom2iu/lhHJgfJBQY1IX3M30SD2Ei5Aq7DE93xAgqTEP7ai+5Xi5d08JplXs9xP5EXxY7cApk9R+zx2gQR/JMNEC8R5JYiGWpCexHVEsFTHw8IxmI5fNabHtfnwiap8ChoNEO3B9Y10LMj83p5+7rbZMVofOkdtwOUU+rjATw56ZQfkrFNi8LUy300V/0Nd9ad/Hwz9+Nmx4q1GX2s8Vzcni83CMVPGcf96v1WhKC4bDG+8L7ztsdcyjaVWLKjS2Z198IqFNkgT1uihkcpK8YWKhQKgLTjofIn7mLih76KAwhwvsNl5T6HFpSLWkjB6jS608U9nOtNSSpLvXe02IRBulsML/ZuaFXrTZPE6IHoKeJr33rsX0nFhei3aWO4LPxWeKUIy7k2q81W5pJ4a3TO3DBdGOTZuqDDVqiwp0JVR2fwvV0nouhYa01VzU4RCFcmm0q/nMNCvhryhUpUD7HAlTGPakbrm4IQAjjZBOj6KWcDLNL8iNsIoILWOueL/Qlvydnv2p5x4RqFIulc1uwzzbcqkgCTdny8IVOSeuiqhCQqJ4oXBcQm3JexwMMOngQ3jo3FUCWuiM0V9JpxRiUUVxYSOc4PWnJyfNi4Q5TXpQJCjkC/LaeX8+JD1pxrdcKKp4TmIsFEO8drulxZVJoK2mk0YB6nYNtODOd+eQO1iefio9MkXUAAp5ej20uh19nhM5HkoVsjkJlRwlmqGUCW84TvGZiGBoMrtde26Fn7Is5vxyTOHAUaD47KGyuXBzc3OvCWUjnAuVH+qb742/6XpPP/eogkw5LcMBCrk8mrU6si6hqbQF5IWCxb5STZykUsnCKk4Mna9koAGN7ARBAvfeIzzjoLk4dPT4PqpIDmK7XhvFvfzM7MwMWu32KKzLc6L7nDhDybiLqRppTkpFQ6K0A4e07ebwaVe4g8j7Npst/Z0mioJRqVb0lYLNC3KHc2KlGt1eT9BLdmSO9+ecMIwUltDrax6klRJaDQN6KMC8Hk0HJYoCxleYNOogaaFOR5+nNy6zZ2/D/PzsSKOG4JvDa6/xWJ6fD78gMA5uAqGh6YzubethplWLzZ2hsCABOq02qpWKSSehR/q83ClpAwG4GNyx3DGx66QmcqZqAjyhMNTq9dd486PY1uFBugU0B4VSUXZ0HC0at4+h8kIoQ7VucXfT4XEAQ0JZNGiXoZs8dtdMXCyzm4kBNPTUM1TBpgWIehEmrUwY3KmFpOYo5PUzr5dn3I+UaRIHXei48aXQldfu9qShKFjTMzOjiGZkN31M1BS8PwEbLUqhgEa9gYmKhad8hWoObcnn5FgVkfR6Ei5uHL4/5t6wCEMWBU7Rdxmak5h66tnHkoBAOVmUODpOmXQKDC3MVqX1gFT18pZztDe2k/h3gg0UgMCF+X6qND68QhXChfLOzRSYM2UOoL6nL0CwJLHYnrY2Yn/6CozZOdGESTWRdK40Jj68LZjtPBfIlMW2HCvtOHetoNax8E82t0sVaVJvCF0GRPEYslBI+FwMnbhr+ZwUBMW57plzgTkHfF5BpA558rliXqYqVY2NWobCymcNDcdn1Wd890tTMqZniOvQzfT0tASJG5DzEoJuzrAJGsdvttxQtRBwrolpV4tkUi+8/IwjaLsgCgdEEF0OBBfL1Qe9VvNg9QtHwMzrJfTJRaEKlQfoi0nEZ2NzwxElG8y41MbgLTGRlwoM3Jzf2QLaAyREy2lfAallhm2cVH7WJm4gf0A+RD6vhSKerJ3q3jd3KLUBF1DXSlnSRzsjbQ6p7bAKehJYe1ZeK9RqxNpyHtMGJnEX8sXvhTJms2hw0YQZ0GegYAwVj4dQclEnpyYtOeTTyvFwiiLMpRAqWnL7G5uEfku9sTNyOu3vKdn78MCZhyBIQ8xEavyZF59OtIiZFPIZokwNvbndaqBcKGEw6KPoWLW8c0mK2Sg+kOBFd3CUpZmYGDkFFBpqCmZcwqYp5u6YrZH5cODGMjp5CY2841xOmoVj4TWofQK14wSGdqA24WfDWYoIIkIcU30ptDud0b1kagbEx7N6BoEghCzTad2Ln+H9+BniCwZYDLBTq7lQM2IxRDGik1TWsk0Ubl6bfoZ2snvcMZ4AP8zh7KM6NWXJIvoXBT4/zUxfmkJ+1MCwBjqTvP7U9PTImTREzoQtwmD+bmS6uhQUcxilgV4++5KEiCBARmrUEBxmcxT0p2jPbUcRXOC2swU39IuCwt9x0gjtlcplhWHh2PDGdQL8zaYGPlGZ0OcD2aIzxJ/lpPCaA3P0qpOTI7+B15eEc9CDvsKi8GojpjR1Y1omJpYIFe0bNUCn05ZfEF5xqG6ZBU9cUBtQi0i1e+aI9k8qME3YNJGGKJWKSIa2kLy/wKVCVosRjlK/w4wefYMsCDYF3Mz3M2oggra1tY2Oe/Czs7MygxGXB6bPZxF27iqeP0sQ220JFneurunp1LDdYSIVy1PLyWY//1TCC+RyWYM23bGhyrTQimogh/Qw0c7iwwp6c4mykMrsnh6eNtRVeG1nR6B+2DA+CCVND5LQqelJYmWvlRk1eJYf53hGgMWQKnoXiTJNZHlzLmAAGgrhaNv1ecPCeT8JL737HLFuy3QxxuZX/p2LaGAPowWOlwtroVOnZ37G0L3xiCzCpvO5OW+0n51O10wLkbY0Q7WugKq+A1S6n4dk/IZhF6OOgKQjvOQut8RMSiqcY+dzxqbgnEYoK83nDhqvR/vOr1wzCgId5Ugppx596pEk0Cthub2+FpXOkGDPrCUMUkyMM1HiMabCINlXUyN0lCSBvnDcoRQMOkemWgwjpvetzJDwdMavGUkdFzqIArHLLRwkNErEzAAOLgr/zpBJpoC73L3rVqcjIeHc8p7joQntI69BoRHSlBhAxPHH/ahOI1mTTpl2IronGzow7TaO7UcsbOrUEibUVFqklAMy/S7o4kWem8/ATcB5irCJX/lZjpfzwu8j8rFM3FDzzh0aYaG0WJ+hZl/+CZ+DIhs+Q2g5aVHOMX2OrzzxsBabEs3kAzOblvUpyIYw7JG7z90c6kJwqKl0hWeesjTPkHivQYMCMnyyeE3loxXSEK60XTk+6GBtmP9HreK5Y4kZUKvtaLG1kxxk4b1MJXeVaJAQuoaIxRMY4lkrM0kWr3Lx5StwEvs9MK6mA0cVST/DQk8TLu2uMUcp1HVMrrJ2SSJvXlEKIxJh8gyxnGDhmTV+Vo6TmxXZW0LGLoiBuMnhYx6AGEOwcTx219iYMWQmMaITwsaDwUhg+RwCv3zTpB5+/MsiL5hX20POSQv5vDkuXGzFa2RtkHLjoRQnmw+hz7ojQlvHvSc141SkwMM5cE4Y6UWUQEocU5sUsJBCxdF8KAdPtOMUqlhYRc1gnrQtgMXLWak8MyW0nwNPF+6SLwK8oE2kAIQTQ01C28nPa/cS5iyUNEFcAD53eODhcYd9DHAj7DavG3FxhEImtDaO8C3CxDUaNWmY0A5M1hAj4M90TCm4XGgKJ0OucAYDIg0oVQAPYWeaNUfslDhyUItaMfyY1GNPP+pMFYt9mSDnhxrNuhaYzgWlqpwv6uE5iAjutbPH+Gjc7bSLyiyNATDSAo6XCzcfZc2C/ODok1N0LMzi5Nv1OB6OY2enprw3BaxQKJoal49AEoGBJYwciGLxPZxkqr+AGyNRMA7YRMxLdWjYQErXpSaIxYisGxcu8PtwgGKxKbTB6qGm0AJ4WBhUKQoRx8+IhQIsP4SIH59xLEbnNRk2hRMs6Nk1JXludHjDBNIp5Pt4T3EISH4grE2giBh8Pi9TKij3iWceSyg5TGVyMFnu7I57fz2qtJYgSdocTly+UEK5zLQl1bqF/nzI0A6GsBm5kDtcUF/CHWuYeAAInHCCFoa42a6MGNESFvQwzQwo/CAE6ULEh+N/20H8m/JAcro0CQRcGC83GqOxxU4Nr5XPKgH0JBCvx8WlL6A42Yl9kXjg89GX4c+2aJaIiMWmg8YF4hgopAzBNzc3R7loOYtyuIxXJ6zdSYYUNGooJm20OMp7M09uiKRsuzuIyk0QtMmksbOzbSEI4+uJsogYEcJFXB+OM7GD1Jce/aJsNrHtGj88HEjd5tMJup22EvrJYIB8sYRSqYzSxASq1UmUJ6Y8xKKDYyqf6pA340LRVlG1cuI6XebELbnP0IYTJKTO0Z7AfkfeKBGxXneESAkJC9za0TeaAJoMjr3bY5zqSBi/IoASU9nKjrmpUa7aKVAUXu7+yJ5xYiIk5ELyvzYA05m9rjhoy8vLyGWY5m3ImYpEBdOvBw7st3yBzBnnxeJ2vm9udlZ+TrNFUqUJI22tOZ4MpxjimQOby+cUVnEHVzwCoqqTQJaK0mB8z6WLF0zbFkpm5sjedSda8+Kw68hmf/mxLyX8ZaO+g067jmGvIyZIPmcTORx0iOojRQaGXPoicoUiKlML8gRJdqA0kiJEOHUwNFQqGCfaCV1yy7bk/Fy4cAGLiwvYs2ePecEOH9KeinjgryAdctdzh8euNrtkSX9OEAkKVOMUDl6P/zlew9oTQY8kSWSFtqVQKhSxtramu3CMAUhEJDCeOQo1zK9rq1c02advuwOf/Ohf49a73iCHs9M2XDoyf+F/MKdgmT9T54pcHCfgV+IOnLdxti43bbtlISIXmxrXHEFuImozmxyxiJIEa2uGIzBvwfmi3S+VLWFFTaJMpUgWBqumHvzS5xLyoNu1bQx6bXQb22g2ami36yCLI5fLmFpk4l057RQq1UkgW/IwKytUh7TeoiQsh3K5guGgj1azhYcffhhveet9MgecUE4+NYFiWIVK3EGkPNmDmUNkHjOFicTDRsPIhJxsqubAyvk3OljdbkdmCJ6WLOSpRSioxptmOElSgBZ0OJR65cQyAgmTwPtywng92UDPpIWD1WvXsLm5gTe+5W34o9/7EN7zDd+MhESO7Z0RHsAJDQHu9Q13N66bRR1yNDNmvgwhsx1Oc2eQr+EMNJvUKPSsFW45Pp9JG75BU8DfUROb+bHsXIZhpwSKiaqszKbRr90UfvTjf5Vk0n3UNtfQbzfQbTN+LYgmw1evb+nMtHO4h4yrBZ4QB88jTbJDvojiRAXF4gRKpYoGJL5VviDItdHpeVrTmBOBo9PmcMEIhHCSRdFxZC5if+4+Tg7NQLvbcWpSRfE3QyXa2Ga9qc9ZmJdCtcpkRV8U2vg9J4PcdArG1tamcHZOEjNh/EwQB8JciF3rW4mfbTS2UdvewA03344/+59/gG/51n+jzygJJC/egB7aawpKs1l/zZgsvcp8g6U9RcaUo2lzIoFwX4S7lbtaCaLQViOMwVk5bhKEySeGFWTyTEUXTJspbBsI8qVzq4TLX/zZf0u2tlfRqW9idqqCen1Hu6TXG2gnKF/NZEQkDpwJkmT5YMwDTyBfKiNXKCObLSCdLSKTy6BanRKVaXpyGps7dUPcFN7Q4zfHy0APc3I4mIhZd4n+fVQqEyIMcFE2tjZx9uxZLC0tKQ/Mscnm0oZlcyjm8zh27BiOHz+O6ekZdFpG/Y3EA2Nnzjb9kJ3ajpH0U4aARXjEcZjGsR3HCadz1GzsYGdzDdfdeCv++i/+DN/2r79LGiLoxeMevj1P1xiwYv0MtYvDJ1EWjQkPX/TAsoMsEk5faDja+OAO0P5qw4CgEfPvpEQXjXiS92oRYhTOy6P/QPuukPnDf/rBBANOWBubqysoTzhJYWjlJ5Q8euIcSHjc4chIEDI5qZpMtoBMlra7gHxxQna9Wp3GxOQCElJkCcP6i+GdqjGodpBCd2ATzAdReU82JwDlxZdewksvvYS1jTX9vecxcuzWcOzGVfHoHtz5JUYPBczPzOL06dO44/Y7BOoEZYcLFHbbgKTirsOWSrQjDB2DdnV9Yw2HT1yPhz57P97xvm82E0LOuUyMOUfhW9Cho8Mlm8xQivj5iPtmi8fn5e/DmVVenqZnQAEzDrrSlA6bCqyhqePadNoCkoQRgMCNcpNmNpywqSSVo2rSJb/xKz+eFLLMTfeRY/oysbonVmGYnbGgPC5CO0Q3n1IXjpI8cd0ASOdyUunZXBmV6iwW9h7FEAa+iKtFe0ywwGNvARwYKmy5cPkSnnnmGZw5c0YL0uoZm4NaRQ/ioVKABLHYoeqCIBDhEgkVfHCKFBedCRSmGMnEvOmmm6QFIg7ns0Y+X0BFwsXxWjKyaTZWsbp0Ea+756347D9+Cm++712iRtEfMNNjfLjIm9PTjjy9tJrnlhU1EATSHBAM4WLtEhW5Uw1MIQ/Acp00WSJe+m4NoCSfI9RMoqcnnpwzyKRPVI44XGj3+LX//P0JbVKxVECKnGXmdJkA8cUhmCV97xmeqMXiLjCuuZH7hCwxFOoPMTk5jUw6j/LUDKbnDmFyZlG5XQoMUbrI1jIuZCjz4osv4oXnn8dOoy5HLZIe8mYdirUFNI6a0Qu5YUzqRy/BmYwc7DchFBa3GzrHF8fBsIg7l/7I1NQ0bjx1CqdvuUVJlYjh47r83M72GlYvncPb3/3PcP+n78edb7pXBX6tesMWeWglReZMmXOpHcl/TvlSalh+gKlxIYb8zMDoTBEi8omocZjgiKcbkFYfxZBD80+4QfVMJC24phDsyhwFMQg3vYFmpn7xA9+TCIhPBihmWQJEN9/LdrSjzdBzNxIrV/VleIeUfDkkeaRdBXECaZyZCJia24NuUsSpW+6SNy4MmA816GNlZRVffvQrePXVV9Go1XVN2mYLxQzgtwW1laMW4WLzRS1iEmsPPVLd/n6S+cY/GzYw3isChvLmNE/GvEwPWVxYwVS1iltuuQWnTp0aZfc4ofXaOlYvnsPdb/46vPLyqzh2/U2y2TQtlrbkeI3kwBeflTl5YeacI3rVjoFHrK9lF2c9IyxD8XmAJq6OhRYWC2hRZauuwoTF5sTSzj4tUtkULoOxeyq62N3ZKaR+6QPflyhWywJDJh6YRRrS1hhFKQj7uyGRTbAyQp7jNpaG2fRR2pDFe4UK0vkqbr37rQIWRLYf9PHZBx/AU089iWa9MWJNWrxrFZ0Kl9xWxWLbw9kuEanPvW89rDMzYzEJqkilxxZ3Idjd2TZ2qVenKvNnyzkbIsg5IaBx04034fbbb8fO6hWsLl3AqZtvQa5YRaFcVdIj8TqrkTlIGS1bfgSdUa6E72gOWz7JWHgU8KuhjtSNxgW0/IFlBM2AkZJlSBsdM1HFXJOEuFui1lBN2/l0DFmk6MLxyz/3/oQDK5XzSDn91x6YWbCWFps7ke+PhAM/Ssg0dlxUUHCHh0dN9d5Psjh7cQXf9h3fJ/L9o08/g8cefwxXl68YgDJWSx1o2jh8GQscO9cEjjvbfIRQ7UNpZ+On0QSxIsScGtMMAlrGXiEUIUghWJaZM3iSU6a8fS6DifIEKqUK9i/M4NSNN+PW2+8UM1aOnlivu4wUwqaMDOhAEZMWS5Z2WaQI2wzyNZzRqw3j5BAurmWwGN6akFD70L5TG3EjjFBGpmhJn/Y5ZMREDSyOn7Sikys4D4Fs/uSP/9ukpKJwMk4oUgPk6FJ5WQztIyU0EhvipzG0cIaJr7iQLKnYtNVqK8eayeHVy1t45zf+n/jkpz+F8+cuaCe3O1TpVpyuHUYO1oi44EkT7TjPJXsFRnjd8uG1K6nGBhh4sZyx12yhtcjK8VqJsNlHI7jF38eFaFybjAtHwKb58gQI1jA+J4tmfmYex6+5BtccPmDeL3qkfouuJIFNzLHV7vTiwVjgKPYzgQzv2ahFgmY7lsAJuJNzTY89dr9COdaBZ4NGxXsa8ZGOXEC8xrBJI0XYlvyBX//Vn0zajQYmq+Sb9QxtoipKvG56wNJQBu4GBngkotooedJEZ+QtkqFhD6b0Jx2GXBk7/RKefv5ZrG1uIDUw4iCxbNpk2maFcz7rsYBhm2PhQtWG6chI4o0LpyyYCmK4iJT0XY41d7+WX3YuhVTGhGfcnsf3sdvHfYBIJ3Lxc1TtBZL3c0bu4KISfi2X5eFP5LK47fQNmJmwShBqiBFU6hUZdLgshbtrPhgDBz4fwEqMyWrJrALGVLz5TwRvbOGNI9DvGRaiOfDUcrBc+DMxc23WD/3mB5LN7XVMVSYsC6UkeQqH9h/Bvn17MDU1o52aLVWMJeElran00PK+nabiPe5WOhgE8pP+EINCFc+/chYvv/yyUpO0J60mHTDzsBV6yNu23Rn2OB6Uv1eO2RhyI0+aP4loPyq8J2Y8MJanY+KBfAnpc7LguJMW34f61jXdU9+140b0I0TJF/EDZIj/M+WbR67AxFBJDpbsvfyeDMrFKrKpIfbNVnDztddKEzDC6QtYoa9jzQqIVyszSIoVee6OM3Ac0nhjPooVRXhRorho1q4EKdvhUTYdqePYHBIW2vVg5Xz6H/4k6XaZ5aIt6WN1dVWkAuKvlCLaHbryzIpJUl18xIPOpOTFmlonamRgQJLL4eJmGy+9+KKcLg6e3mGzaYjPSK0ZlVrvsV1kYU+kN7ngI+ryWDWE/C7PiZvN4mJzZB5aOcGBJsfE3VKioSliYcMsjNvzEDZG/0aiMEdIi6SEQxHFUkVZQC4UVaS0U8YBGAqiV8jksmkUc1nMVSq45aaTgobTXpJLZyvoybLPo1IdY+2qqsRLltR1watCtEPdQeYGi9DLtoQ5hTJhgp4jXrcwL/UXf/RLSqdQCsx+GrbLeqSwlLcAACAASURBVGVKEFWFpQB366t5MzpYVD9cSEuRplApl5CvLqJXrOCVl7+K7Z1tT/dZxobCwCR/qGsuWDgY8RASHKFK9PAt8xYPZ7nrFLIeUlAABfprt7CyMoMBQ5mITp1HF5LOz47b43FPPDJc4dD1B8zpm2PFCSSOzs8TFqbJylcqUum5gvVqSWjC+kaUVIHgwHqqsFxI8zrsygGeLGXx7ne8HSxl5D1VvizqtFWrBpUrtJIxTswkBMxqxY6SeOcAmh/i0qy/8dmiPs1dFqR+4xd+ILHuOlbiQlBBXQdy5FSToGDeLKmzQqpUOG/0YpHbvc0EXaFBfhKl/dfiqYc/j3q7hW6LjpgJCz9HDjZBei6MFtE5zrHrAgkL7jYHH4BNCIF2WYQXopsx+LTnlKOUIZ7kxQgeesX1YyG/NpwLTRM73cIWCwNDy1CdcxMYPFxEkiNzp4wkYzufQsD38FqCdj3lmvI0roiVFM52C1tXL+H2G6/DO9/5Ts/W2diJZ/Mlb97JFRKUsZKrCKtIkmDVjsHYHoV4XxjLqRv3PIAcRQS/9cs/rG1n5D9ic27nvPoiiuRMzbgO99KfiANbrR0MhxnsP/12/N3f/SUyDnZQOxiNyJiTzDoZB4w/m80Sb83VdYRtob7DBsm++w4Zt62pUH9qCUVfg8O3/HHs4PAFIqQLJ2/cRxjH2GMMDKG0WxyNE1qo3LLVUTHTx8RPJl9Chg4se9Kwhj2VQb1hiR9OGGu4FF4hjXTSQ7NeR7u2iU5tE//ym78JJ48ftbptItxO+DAGi5mRICMGrs4oRxx4gkwwGFUl6iRDiMpkcxuVNJFdUzLlv37wP2ixVZfsZD05JE67FewmgMOACM5vgP02EH4uwczR2/DYc1/F6tIr9neVsUTLJ7NrDCcaDcKmJDdSEMx+M24OdR12VWqIVZNy4v7/VYzane5lWu2MIUtc7FDX4Wz972x0/C7s9bizpmuz84SXB+k6LlhRCWI8vDzSuRISpRfJiSvK8TThNAezXGE+voE+bWmvo2Cwtn4VrfqWHLef+g8/aowez9eP8geROxBl2KBYsW2UhevLUMlNUbxOyNXyF7wW7z1OqwoMI/WhX/mhJBZUgIX3BIv6qmBXWALe0pPuH5tXyf+dFvLH34L7P/a3SIYNDZxMC8F3TMnxMwJDDPK02m4Lk0wN79rmcFSsPHfXWePYYkxRQWnjME63TJbHcKGmww+I3bp7bbNv8dz83jJ4RpDQriSvzZEv+QxU105CMNvpoU62YOYuV0A6V0QhVxSIwQVniljz0++jTnIGG24NE2ytLmN7ZxXpwRA/+1M/6R0d6MgydUmVbpskiBARchl2bhiZxeduucliCQfWKckjs0aNOCTjN4/Ub/3iv08YQrCaIfhhu2GPYa8RAoUDZ5JvO55aodnroDZ5E557+CHUayvyUoOcR+FhJ0LtdudHEVMW0N8xcgFDMKk6955t4i15Eeo7FkEL57zvWLyAH9NZW0Q5bWMtu8a97XD2wqEZQZtj8Kny7EwFEqgcYdVWshTqn0V0NqHuw5C/njMiZrqQQy5rxREZr4ztscojGQgf315dRr2xjnwqg//4Yz/ila1dLSQXJgoNZJfFErW+K9FKLNp1EBs3pMyRNufnGZpsXj2/mgYGUh/8T9+nKk5WPoSBskm3zJDZM8szx1dzZAylYrhEqtLmxLV49itfRLOxpsExqWDCYzsyYL4g9wVRn5+ntgjnKHZbnoUEASOSOapWGUZb4kv23MEVLTpBBu4cx8/HwZH4Pr4K2Bgj/MeCh6NmKt18F4Ieso8Ou45/TuPwWD6XLig0Yx6/n5D4UGLnS5RLJEZah0JmyQrZNDZXCRevo5jJ4Sd++AcdLbPuipayNAdTIIwDMOGoKUHkfsS4mQptFlrMwBbWirtW5dxxsWUPnPX5tZ5qEP/dr3fyn4Hz2o3suNDpY/KGd+Lxzz+AixdeRNY9VO5wMk0M6SJD1CoUgjhnHja9cgM1DB40ocupoJBCZa42Q6qAT0cPOQb6K+4nNjDWqoPPFQscKjoctPHnDOctBM5UqAmVFbfbDhnVTHmZrqIRvx93eIoOWybHDJChXKRZFyc1hiafvdVGIZfG9toyavUNlHJ5/NSP/ahrNIIO1Epm7zkHyi94nbnh6bYfd5MlZsi4uagNhNx5HkB22pHMqC9P/ebPvz/hgKluwhGKna3p9fAodpOBdmzlZIxKJgJanT5Ofv2343P/9ABeefZRZNJUw6wVtvJdAhGhsg0T52TKuzDKMLsVhN11hEwqyEOvcDYi2c8HkkMXjXr4wKL5WLw5WgDPzH2tGh/f9eO7elfr2K6WgIAolJVARdGinM+BJzBYo6XSHysglLOWNgHJ5stC3bhjudDKQPXbqG2to1nbUi79R37g+1+jrYLepDVx51g5ctcsMUYrLdrtLxsmRqGqGEAUxF1QSprhN37ue9VAx+LBcFJMYsxT3m2foR3mHYXDzhK9ajVauO6d34Gnn3gWzz/xJXQ77NhgHuHkpBXDGxZuVRoR+1kmJ6V8dixQ5K3lhHmMKiKe57HNSfOiAW8UQGecjk/kt83W72a75FX/bwraQ+XLprmDE9/H5JFLxvdxh4emkJD3jDOnZxqShWPv0SKl89o8SOeQVTtN443xvflsVqyXTquOublZfO93faelI51PF4Idv4tx8e/jYwuTE8JhPpDVltNB5L2ClxDzl/qVD/w7lexavbEjVGNNVqN6kQ8RN+CFFhYWwBYQxWIeSSaHzuQJnLu8ise/8KAexpy6IeYXZ71wwOyWhVKmqqimVNM84lPvdn+IQgOOje0raYMCD4/sFheedj0ctkhphoqORY5F3Q0jvZPDGGWY4+JzRQgY6jBaXkdnhQA4ct5zRmgZm+8RIVSM7w1o046sSWPSnzVGSqrLxj/b4udff/11+OEf/EFfbGO2hJNq/lHAqJ5p9HZlaTmHDDONYxa1cdS6mltH56h9ogpUc/BLP/OdymczbolYkzsnVGXknMnbYq8RPvSo1ssTCCwZquX24NIO8MTnP4Mrly+OgILyBInwjEENFQpEzXZL3hrTpq2nWBD+xu1sOGJmUkIhW2Jf2ACT/DExY4iZdp+XvgYuEJM5vtPDHkc0EL5DaAIrKjRGy8jR89BHvVy8dZeySwlZKabOuU4K1cQxy6g0R/dXjqAuuPRd73o3/vk3vHdMjTMnb+2/FPJGaOpOqXnf5mkr7aww2Xh9Rllwe27fjHiC8WypX/zpf5swSJeKYTG351S5uATuc85bjpCF8bEe2u1jmlNNzzFVwvnuNB556LO48NWXkMomyInUDiwszo2AFAvx0t5vu6ydHdpDu9ix8NiNoY7DpBAXd1/JAIxUImGx1N5uY55Q5fE1JinEJa7Pn2PXCuN3vH40qeS5ec45FtxqoS29Glg2+WEquqcL7tGCqWAjTrCXaTTwEVU6ncKHPvQhlUiHmRPbhw7pWBp2V0CtBp73NQ3rFC0nMHCiJdzeL2a0+B45aSwf+In/OyFXiv27SbpXB6IRMS9tOLSyLN7wLpIQUYutBu9ZdIcJznXm8ORXHsa5l55Ft99GOrHWUlNTE1LZFDcurrzMPqE9a0jL3msGtJiHHwAHB8hdoqY3rE5UV0Dz3G3X7qpxg3stsRI7OhY6zAavN55wGXfUYnF31WhMqoFIRtm1/IBSvS41I+dJZLY0uh0nGoYdbvdUkkP1ru5L0XigVMQHP/hBoYCGVnr1ihMTuKjGOHGKkYeD+tmTM0ZiMAatSIteVGkIk7FUhcwpu5hC6o9/9/9J1HzVS2eEgdDekBJM58JPGMhmmOVJI3EUiQsshIv9vAg2II2vrnbxwvPP4qlHviSCvvBqVmeW2LzVPPKYVLOPhhoV8+wRYrxyld96OBOLEwLAWnH+jTtZsbtHBru7w9E9j+3Gw6zxRRy/7tdqgLh3CA0xcj4rd4xahgRI4YsgJ4222Om84deElookje1QFjQaF+/EyWvwH37sx91OBxXZulOpfwrDWmbt1FLL1HIIp1KqhRyGHWeiOOql4zjU9M+aBFohgiGRCls/9td/mBTLRWTUSwQCBZKEKTfr2zGi73oFQ3qw60QpNEmxwRtj3DSu1od48atn8ehDD2B1ZWmUiy6W8ihPGJPFvHEvuAtb64sbPkOYknEHSw/oD0xvM4SGYyTGzOvGZHxtDB3OllKKXgfN7yMBIgFyGz+uBew6VuhOSFRC5zy34I0x2aNIIW190MI+mgOaRTIIO2u5ezstIY1f//VfwczU9AhsspbfFs4JKQvbzHvGbg/AhbaakYznrpW/GrP1u2RM3ziujVMPff5+IX9q0KL2y757vGwm3H2Lei0nPY4hy6HxdFo/yeHxVy7jSw/8Iy6++qKpmEwa+VxWhQfRp4XccF5OdUjFDLpt6xca6pkTHs1aaU85iVTz47tw3KabJTPHJUKRWPiv1RKx2/lc4/cct7OKSZ0gEOxPYeXBb1NDH2eQuhYZjzLsnhmFWeY505QbCklG7Xd/93fjDW94nXPw9FcRMGge4h7RrYmXFzVpnA3rfPQe07DUKS64chIpcKo5G8rsGcnRk1kPP/JgQk/R0pykYxqYMALhnWLbb1uXWz6keeNx8k5KD8JS3VyuhOcuruIrX3wQLz39+AgUoNQyfjS8mXnznpAhkeDTAyR9CxnGqzPi4aJOy0AZE7RQw5EsYYO+r0XG4vOhHcIPCDX7tSp+3L6H4IzfS8wVz+Pzmv2ehakhMCEs0cFR3HkdTZHHgYMH8KZ77sGdd95h+RWRRUwTRe6BZkkOn0cQ0UslFt9Ewtil9PLDWbOMJVG0XWbqeMtt81E8qfT5z9+fsBMv7aHVPRmfigNSAl0XIqmcRXQseLOeXqxgZH5a2DbhTZ2pUcCVtW18+nOfw/NPPKLUpXUpsm75LMfhBLJVRKdjvcJZE8XidoUT8jDNQYtJCE95F3TZ7T8mQqEcOscH8plRV4TAv3fBEXOc+IpESahsmYgxtC3MQGiPuHcsfpiC2P1a9HYfe/fuxfu///2iHhsM5Pdy+rAEMG3PZxTh3TGxr7uIEuwU6Y3reV+WRRlgYk2AeS91qnAiYtC2rJWJbRoCQcIlIivorcVSD372kwmzVjqRJ2vdh1l7FQDEoGt4axSuST2pgsT7blLd+SEtjDFT6QKefOUM7v/E36Fe2xoxIwnAWO/SrOq2u11SZ62WizaXLzEyHXCJiYoJjh0+PtFy1EZJGh65YDZzHIXiIkZIFRBo7HK+N8xULGjYXA1ojIgYAjCeJ45dd8cdd+DffNu3e67AKjZpQ6PG21SpF+2JXGmYugmZVW8QhwgnkjtcvD0nDHLhtHO9k4L5GAyTdxeVi22JKzp0Rhahn0EBoGoX+vfpf/ibJM3QqdPWLstn85icncYLzz6FYcIwjJBnFXv37ZHtaNU3MUgySGVYrZlHZgDkK2wIYwxPqphXlrfw9x/9G6wuLwlDZ5E4ww+q6Xqt7g3r2BfNeoMOKInOlFEI70kRIy8ECXG3VktxtZzH6LliNnZ0ksAYOTGw5JjIWAC+N6jIdoSUYf29riF8/G9CbdpGCQ5f/NAEHCfr2n7mJ39KY2ZhgHqjD/qqTbfEhqVbWYynpvYD48rzFa1GuLBEIlUbzoZ9Y3kBnVDk7SrDbBCNMzqxaYg0mUHhs+ikBeMPcvz0j4zFk0Lqr/78D5Lq9Ax63bYkgdX611x7Eg/d/wkcP3EKi/sO4+WXX0Q+m8aBw0fx8tOP4/ipm3DxygomJyZw6dXnkJ+YQc/JJCwiT+XzuLzVwSMPfUYdE4kzVCtV84QdoCB0yvBASJDiCqtdGn+Zat/9XahNBXoKKSJDZHlmkiNjUUMtj9vmXe+eMazVnekeHpoY08N7sPjC8prjsWqo0sgw/b8/87OYqU6pw7HUvldi8Hk4FoavfFajEVGT2PtCg9gzMS9hVCRRmdzzj0NtKDChUaTxmPpVBMDuzz2rvuUpB+xVquY6lofv+r34GYFVH/nw/0hm5mbVe2t6egoXzp3DnXe/Dl/8p0+qo++RU7dgmcXvVy/h+tN34IXnnsDJ625Coz3EwsIcHn3gozhx+s0oqEVFHfv278fTX7of5cM34S8+/GEsXVpCPp9RO6geC/ac6cLJ4aFkQnpiQcc93rGFJl4VvTsNVCHQE0wWS4wYkGKCQVNjDppXcnqXYOamJQyBKbN6xc/90G7lzus6Bz1Sq9EiOrEMHR1F64OSYHJqGj/3sz+npEh446ERgnI1KgOWX8IerB3tYIJNpkms0Q0PYlPNupMuIoyjsLIxACneuXzBKkM8VCQMbfQuo25Rm/R40kGpKN+l06xbXThbpdCGs/PC3MI8dra3MT+/gLOvfhU3n74Vzz/5KNqNbVx7+xsx7PZx5sUnceTkDUpyFEtVzC4eQnlyAk9+7mOYmN2L/Ueu02IfO3YUjz7wcUzuO4LOsICP/t1HUaMq8dZV9DKFJMkeGUU2asis04QdTmbVIl5HNebIjHunEarJ3ku1pcSQMTVoFY2aPDXX3c1ta4d7VYWS+4RMM1YjxYlnSMjvdz16i5F5P3rXFk7mVaX5rne+Gwf37hsldsLBJFeNY1LbixZPTjCba9i4naQQfk803+NX7sDwJaiGubhsTBC+C7/yOjqZIA1t0si9B6N0e3vHyCNk/uq4Spbx9pD664/8fjIzO6u2FWxNwSTG8ZPX4crFC1i7/CoOXH8bFucW8NzjX0B5eg6TlUnUG01cc/I00rkMnvvypzTA46ffpAXau/8AXnziATRrNRw59UbMLsxic2MLTz76EL789BksXb6sXWGevrMynMkSB4lG191oWZl4q0h+jhQqPgiPfeAujxYUVu/sPcZGoIsd8Cq1SJUfdc1OiJQqde+fAIXh60Md+CoMWiR9o/bypTiYcbP4vEAubQ1riO2Hz3H06FHccMONygqye1TUG/EZFNuzOW+vp13ISwVMSgRRi+LnpfCrteMsqgcMhZj1d1w0CZu34OTOpkIzSDnB7MysasXYnSoO4su62Uj99V/+j4TF6LWdOqqTVaxeXcbhoyewvbmGK2efw+yBa3H0+LV48ckvoj8E9u87iq3aNvYdOI7iRBlfffJzaOxs4/ANd6HEHT87iwuvPouNy69i7vAp7D98rR7wxScfwKByAB/72Mdw+fKyqb2BdTgO+0Xpj7CEoQapwnzIyLZx8Ny1Ukm0/Q5YyJN2gbFsmLXVjOI4LZYxHV6T16ZajyTQbjLFD5rLG7NVbBSP7y0c9DCR2kQcNW8G7zn3cNCII3CcLHZg/7SJsp1lwrCM5nHYbSmKoa9jdKs0+sMu7Y4EgYe55Qs2N9T/1g/V6r7Y+ULOGokjjZqKKNVpiTVfbPbXrKPJDlM6Xbfgba0HSP35n/5uwqpEa59cBM+Xmp1flId86ZXnUJpawPEbbsH5l55Rw/mFPYfEpZqc2YuFxUWce/ExbK1cxsTiMezZd1iLvXzxPNYvP4t0YQLX3vI2dSB89bkvoNnq4vMvLeP5xx8fqR9BmNHPVOwV271c5JKfFMDfaZFzu0kaIWV+Qq86D3i2R4APTxQKh8lLYwngMOHCtKrRjiyhEWaBqcoAddQtSr3COXF2hgfbVZl9NB+DZT8sMOQiqZuTzibxhgEOdFBQeF/ZVPfCC/kSDh44iONH9mNl+SoOHTupnnArK1dRmShhdfmiHK3DR67BytUVnXaYKxZVhdlt1sVJLzAbmStg2GubZnNIt1CqamytTgvVShkNP6lPWolz9Vd/9jtJvkxyoDVutzjVmrGtXDwnZujJG2/F8tIFbK0sY2ZxrwSjOr2gU/GuXjqLnaUzQLGKhYPXYnZ2Adubq1h69REMBykcOf1mdUQ899LjaO9sYjs7j4985K9Q11FN5pUyZOFXWtp9+/Yr3hYzxI8nZlTGn6lo1ZMz2l97VaaFFlSnFk7xWlJvcaY2QaOx46oihqeaFN3XF5+2UPdxhzHUvFKq7jCypo0aYZzUEeDLOFizGzNb7xQV5jmGoNjeyZgEnt56772YmpyS8DY2LmNicg7XnLwJly+fxc76KvYcPIyt1VVkEx4ydxUz+49jbn4R68vn0ajtoFouQIfjFLhBymh3Gug0a+i1TdAIdnE+Un/xJ/8lId+Z+LUC+X5f9pDhQH19BcNUGvsOn1B/tPUrl5EpltUMNpUpYe/ePdhYX8ba2efFtZo7eB0W9hzAsN/Buee/qCMo9p28HYcOn8CVSy9j+/IZJOVF/PnH78eFM+fQ7Rnezfvu3bcfh09ci/m5eeRy1sEvuv30O9bnrMQDYZx2LBXrP3Px5HQZqXrk8Qu8oPCy+I5xrjea5zPy89FFOECX8URKNKoNgYmkCSnBStHGkY9RPDiWw+Z4IlY3xGs3JByhdrLhPF/T4F8ybCmQxw7OYX7vIdz9unuwvrKEKxfPYe+hw6htbKDb3NKc7T16E0rVKVw5/zLQazGzquKLfGUGM/OL2NlclZlg10rejzSpEos1//T3fzkR31nF3XYqnzrRF/LoNJuC6fbsPyJbsaZMFoeWRbZYxsL8HkFzK+eeV0gxufcYFvcfE3l96dXHsbO5ganFAzh6/BbU6ptYeuUZtb185lIT93/606jvbKDR6eOHfuKnUW8P0B9aX/B+t62meYwfCXiwebwWiIiR0CnGqhazdhjX09apM7E1j+VxVRFeqcpFaUMrciAwRE1g6VaDaMPTDR5XcMnioNnIkAmNU7WqMWIDsKHNpcPJ8NLOFfXTdrx8KFp18/ddnnnqfcfl7XtmXGeSqZdMTxSmQwcP4Z7X3Yna5oaAm15vRwvOse+95laZ3NrmEmqbV9H1as7yzF6kszwQponWzgpSgz62eYpvZRKTc3uQ+uPf+/kknS2gQM/RWQ18eC5Kp832WAkmpxcUpNNpo//KTZUrTmDf3gMCA66cfQHDfhPpyjwOHL4OxXwJaxdfwtrVcyhOT+PaU2/ULl8+/6zUYbtyBL/727+NlbU1fNcP/LjKaLa260ilzYwQwKF3WSa/LUlEqqCw8RpimGZJY2L/MaYQ+xh2efRCH722N9cbU8uWGrXr2kIbYNwmsqdG+EaJChiWX62Az1pYRIYvgI02QxgnSQaiJWqSw7KMcdXbTYV90aXJEiZ23rbF/vZ9HMhqHRSkPVRTwTH1UC0V8N6vvw95HajXQnNnW4zUvcdulTlbXzmP+tZVdFtNadvS9B6Z1+3NDaBXw9ryZWvik6RQnV1E6g9/62cSNpnLuo1MeUaF8KBaMOoQlylkeUh3r42GmCZZtdCYmJyRyqfdbuysI5cvYe/hU4JXV69exOblV8XeYAjGU9uvnHse9Z1VzB64Dn/2N5/EiVM3Y3pxn45n1IEvLEFVKGPg/wghEzrURSGbt3M1szxkhXGmgShpgjE89LxnXYLZs7TXZN6YkGRXNdGKad37p9dPDRKN9tSvLE+wYjCCcFlxysW26CCl7gahBfg7zoslM6xsmDvbnD5r6MfFEA7gvcKjC4Oa0PF0AF7DY2p+r2ILfc5r5HrWFLA6kcc3vOPt6LcaGPa7SJcncOyaWzBIp7B+5Ry2rlxgcY5M4fzB61EqTmCYdFDbWMba1SWFqRSwyvQCUn/wwf+YkKhAiaItYvsIhhNsXqf2Dil6x1UZeXYopoqU9BdLKFen5KVurS+hV6/JBMzuP475hUX1DVu/8JIWYM+J27G4cABXzjyPVnML5YlpPLvcRXlmDp2etd8S89QXkhk224l+aqA7TMzMyXazl6p77oasWSUoEyqceDaHS3kbCi4YPVnZzYT/DeumqdFB65HedWKAWlzJy/YjLbwgYChTMlCOOrSAOYK77BtpAbD7RFvevPkJ1pGY17TkhrUXCdqQBMd9iPBfDDJmVScPaAW+5Rvfi/SgZ+ZtagYHDl6PHoZYv3IejbUr6LGWPJNBdeGYmgT3ei1sXL2IAR01xuoTFZSn5pD6g1/70YROGNtIkFrERVZK06sp1JvDKx0M+7W0W5LKYnJ6CplcEd1WDTsbqzqFoDp/AAcOHlEP1NXzz7PfFqb2X4vZvfuxvXYVm8vn1PZyYt9NuLTdwOb6ttAuJUl27LhFmgp77Ta5s7DL6sO5s4lghSMU5bWMyyWILhQcL71QCpESFd6ey0piTCtQGFhTpSMn/WgK4eXMoHmKUhAoETcJgZU80RsPx5Dawzh1LHw0UkR49LxnOHcBgYawBFrGnyk00gxjPVzlHWWzeM+9b0C1lLPqmvwk9h44KlOyevkVNLau2rNkM6jOHQZDO4ZrO5uX0anXrCd8Lo+JyWmk/tsvfH/CKgZCRTlWIFKUrNLLzqygM5GyKkURERkzisGWQ5GdFgoTGPSaaNW20Go0QCeBi02MdvX8CwoBJhaO4NCx42g2a1i9+AobV6By4HpcqvWwvr5lZaaqELWJ4iIrJednafG+ERLxIQmSiEbknCum9Pi5qNfm7jOWqhMTiaDpyGg7tkH88yGUk9fnlIywMLA7sG4S2ZQVshMjUNJDXYzICvW0qHvhhoFbXpq7qOskD2kYp2AFeV+dFb6mTCcSKiGMwaAJX4Ff3/2W12P/4qzWZXrxKKbmFiVcq5dfRae2au23CnlMzh9BuWTtvzdWz4JUETmZ6Swq0zNIfeg/fXcigqHjyAmbzbK7AltLyzYzCc4qA3c2VFCQIJPn+ZhF2XpOXmN7045xqlaxsO+ornHlwsvoNtaQKc7iwPEbJCjrV86i3+mjtHgMm/2iuFRXr1wxRMhPD7BeXl0hZOEpR1ZMRx555YUQLSpELz5Uk9eoBGU9eJ4q11RmxOKWnuTCkCnCyfDzNpyDprM0WJbkvdA73ThegpSfFnLUbqQww05D4PUUQXS6fta3lSSHLQ8nLnZ34O2RJo0jKFyVuYDasVFxxOV77nsD9sxO6muDMwAAIABJREFUSkUX5w5g3+IBLeLm1bOobSxZGXRviPk9R1GZmsH21ibQ21I0pANwGx39PvVbP/sd1AFyoDgwNokXu8MdDJaeplM5JDnLVVN9m9NCmnAJ7A+mZCNVx9YWUrk8Fg8eEzy4fPEVNLeuIElP4NgN7kEunUW31UV25iBa2WnVSa0sL2uRGA9zt6lGKTPEsD806JBN5ssT4IlEskHecC8otOwWQc+a0Kd2ijxj8uDN+7bOidYWK5L+dK7YYpMTpaSHs2aiSWyUNxGv5vENwx6dKPY86arUNpoXtPtdMw/eKIj4dajigIEjPx8xdhAX6DyFoxhCbQ1sR2WaEuy3vek2LXapNIGpfddgbnpBuYzNlbMYtLcUmRQmJjE1sx/FiSo67SZWll5B3rVVNlfEgIWHH/rAdyZiOaQtO5RmGwmiUZ6xIQKsGmVWJqZTVmzOXaiOPEWUJspuuwaob22LZTo9u4Dq3CK21y6jvrksFHnx0CmUKhWsXTmPZn0HufIc2qX9SkRs7WwpyU71yyOQAokKtRyn+ubyhosTdaKNJVOTqUL5QGOlM2Ez6UOojIZwqx+uqkn1BjTMGFEzWJ8XClZeuLLial88xqqETOkEqTmfU5iUVnXnyrxpO4SdziCzXJEAEVbujFad3R1HZYjM4Od8e8M6TmQc16gx+CE0//xdb0KF53snKew7dBIL83sl1Mvnn0ONNps59HQWE7P7VRde21lDNunIBxLUW5kStzD1X372OxOzOVb0zZBLaFTBHDX2CleaMLFQQkcTqNk5Y/Gy7IF1sx+q9zYHWChXMLfvIHrNbaxcflU2ZfHIDZiZWcT2+pL6irAJfXfqGvkKXGweDcFqTsbtUaHoLbSlVjmZhFE5JmLcUc9katGQNf7nwgX9iMQJ29nBJPXKEYV5u6fvMU896HfkeCrP7nGwbDeb1PJ0wFJeKBfrzsLDVt83liA7kKJkhjtYTGTQOYquhMYPYzLeqFfRwcJy7pGPtwaC8iGcEcr+qd/yjW9DliatWMb8PvO4eZrP1sqrqG+tWPuNdA5z+46qgrTZ2EK7tqbjP3QC4YB14hWkfutnvt11hpXQBhtEh6MzvFExALnZWaTzVn8sJiSTD7Tn5K3xZKC8nYqrcy1KE5if36sdtXb5FbFVJvccxszcgjr4s3mMSIvlEwpVOmxDUa/LuYlcbuDVlvWx8ETd/dkf1Q84CcZKwkXgJDsi1uq27TQgr57kLlVhuoTaGTHe2sPOv+buMz67cs6eCrW4Oiv8nCRJOX19rzrReR5RgUJBs8pSMkeiEQl3KtOl7CYch89F01i69jI3znc3X4MttqzDAgWHWmeyMoH3vO1OTFan0RoMcejoKVQmJrFT28L60lfR7zYFnKTSZWlT9UEb9pB0G1hauiRNUixPYDhII/WbP/2vTY37ohqldRdW1NmWKo/M0OCpFFUYsnho1geMks42URaCMITIozI5h8rkJJbOP492s4nKwkHMzC5qR+6sLVviYvpa9NgxMWV8rJ4X64fHysmXSiY1iBAn04I6e9MSGNwd3Fl0jnhdlsFGaSwFNc77oAqLuF2qUud/GeOFcTX/RuFmbRuJAqq58lBqBIl6fM2TiMPmmrnY7aYcp/Ba41w3LXQO++yVZJTrqLSMggdreGMLLSrx6IjqtDTD1FQV/8c736S5nZxbxNTsfoVXPDu7sXEJnXZNglyd2oPK7KLYNIxqCKrwpGSmr3fqdZRLk9zZ36Fi/MjcREDPiVD44+CCtX5iC1s/c1pnhDA+ZjuJtJrCMUHP9BxDNoIwk/ML2GKXgc01ZAtF7D10UiqPP7MNZmX/ddjqG57MhHuj6Uc9DW0RR6GKdiorTzpIuEu7hpUTEVP7KLbS9J7oXLxI6PBZomCdpkjtuHg3jdvqrWk+goIbTQLkoHq7jvGwyey9dX7UGVrcJN4dOUgQ/MoIYLz/anjaUZAoCpXrU+5sgwGN2B9IG1uAc17vufs0juxbtM2RLePwsetFaNje2cTm1XPotWqoN9uYXdiPdHZCm6DXb2NjdUmhqDUw4Jrlkfq1n/y/VJ8ttTFWlmq4MGucrMsfU53y1kX5zWHo3QJ1oEqprF1ON39re0tYNosGipOzysisLZ1DtlDC/P6junnS62Fnex2Ti4exmSygM+Ahbzy1hhMPdFpNLabSrCsrQsbUUbHfwvbahtSikKiehU089ti47XZS4Hi1pdGS/MSByIJleaotbbkVHhi4stulwPhscYCLV0+6lpFH7WQ/2d047H3sFEE7etF4YSE0VmCw26dVrFvaZTpq6pC4W8BHLcCzWk7fcho3nziMTqsmBK5QncUij+FImGhpY3PlPHrNGjvJoDqziInKnO7RaO6g19rRQQHUVKRIsX9b6hd+9F8RNbbzPoTC++GnnguWeo/KSTVbpUfMHizehsIPbGOF8GR1Uk1pq1PTlldOpTAzN4+rF8+jN+xg76HrpHImiadfWcLk7CLWM3tF9WFMScePue0aKTU6M2tTCRFmgsjk5RENje0dqXvBlElw2g1vHq9uDApSLLx2ZZza5+UycVipOh6JyMIODFGf6ScI+yLuxskegqrbgrFbuctD3ZN9kuJCC//uW6/vsb7qTGqIaDFioBikGqzVfDaDt977Nhw5ehS5BNjavKjsI9X9/IETmJyeQ2o4lBrfuHpOY6YWzZd4tGNFgkuKdrOxiWG3Y4fJcjMih9Sbbj2U3H76JuxZnEW5wGMgbGcYsmTHOUnL+JlVVNuSfB4xIftt8CV42MpE2equqxXtNDam3X/oEFaXltDpt7D/AFG0JiqTU9hcX0OhmMdw6jp0kBOjIzhZdNSIVtG2Moxpt5totWroNNtqkcm/G1drt8JDp+xSCBMoHAv4MXaptFLWIFYdqRB9x7UQdppwf2AkiqhBD7ttTiNtOyfDW2RFoTyv56Wz0jKEPcWMTsk5ox7ghomW21UeLyV2ib2OHz2Kd73rnTrakX7H8089La0wOTcrz7+2eRk7W5tqaLD/6CkU6FUnJG3WsL58Fjwsjru2VJkBUkZy5GIPBy0Mve1GVwfDVZC65YYDyc52DZ1uH3vnp7BvYdKci2Qg7teeuTmxKKpVghpMORpRwFgtwqasFbPjuJwoeucKHZIheEYlJW91dQULe/ag3e6iPDktQiL9vurCYaxiHgl3sLJUHaUtZZO7jFlbaDUbqO1s6G+M5UmOCOyZE0Shi1NpFaOn2bynjEabJTNZxc/WoZ+JClOlPG6AgsoiCNavjRIgsJpoU+27rUWCjCDVOxiiFGd48z00H96TLCNUz2JrhWR+AnAqm0elmMVEtYiDC3tx/fU36Pip8ClUxpMCnnj0EQlloVpFv9XC1tplgGeDF4ooLxwWKbRR20aztYN2bUtzRH8qW6yiVK7aCcHtJrrtJhKCQATApE2ySH3vv7o3YTqvR8eDXYa9+ZyqCr0/mb7qRAErLdGBLf2hFnl6ahJ79u7RQSqGaLGSgtUQrGe2Qv04TqJa5Yl5fRQqVSFOxL6LE5PoVo+h1UuBNWeKibsdLQ4dL8boGxtrGrg87xbP/zLcOcJEqWOPkYm4EeUSEZD1awXrrM+QjQfAqgyHKFjBCIUsT2ZhgEgDNGEeOAU3OxbZ4E1r0MvPTfL0PyJnLhhWnsPr28HqFMZKtYo98wuyvRN54hCb6LR64gIUJmZxww03jLo+EKmjKfvyF76AieokSpOTWuy15fNqbstoZ/bQtfrabtaxvrGiEJbRMdkz1akF7XpD69qq8GFYxnFIjdP3+vkf+iZtEjZmV6rNCXW0wZwk4b7qprRbtald5z1MlaPyqg4V+fnpPTOzM7j2uuvEqCAIYIOwDj4E7SNVqQashTkkU0f1WcbqFBR+JQOD8XOzuY1+u6OfyaYUB9pP9RXgIgDD2leJBOAn7vCe6YxVTPa7BF94CkBJlaOBgKnvJ59HqVbadfNfmC3Ty7NbnFUlJzy2Vh8G92tYp8Wdye4Kx48dU/NZ1p2RYXLoyDVoNxs498LjSPptEGsvTC6iNDGtkwXjUHoWPfL5udiV6pTCrPWVZdRWz9uclWew9+Bx45HvbIrlQ4iaY2r3eiiXp1Am7yCblT3vd5mOrqtdds6Zralf+YlvVehFhUz4Ubli5oVVAdGjhTJnw20UmV4CKFxN8fd2Gp1liSIG5c6k/TLbbwT9bsfO/5pfXJQ22L9/vzx3kh6Ge06LVkumZiQSqKLIrWq0ttDheZs847vZsF2tQ8GNzMAXcXsKJl+BSRND77Pdh0jypFsVBcwwNOFY5ZiNjk00Z288V82Ja+zU7JgI1rn5ATlk41II+PXUtdfhmmuuwebWGmZn5zAxUcX66jIaNfLF+rjx1rtECrx85ln0W3XNyfz+48gVyzh06JA0DL3xKGp89OGH1fF4Ye9BXL54Dq3NS1aDXZzGgaMnNY9rq8syZdnUAM1GU2dwZrLkBvoZpMOekk6N+rZiciat5KP815//ziSqIuwQUivoppo2NTeCeXczSqPOu+pY7b834ELagQkJP/vLSkkNmaOU8e+0pXSoKCjqMcJMenU/7nnft6Pf2UGjZWgWsd3hsCe8emdjw8kTLQmWtWvmrjWP02yxOZb8T4I+zzmhGTFP2QiJKrLzDglBPxpRguh3iOPmJ+QxqZKy9GppghqqjLfde69ds83zQbMoVytaTFasVqozow5Q3HV0Lq+/5Q70Wh1x6evbV6U5D5+4VZNPPjmdVDsdyMptv/DQQ5jU4Xd7sbWxgtrVc6i1apicP6bUMcda49mpTXaeaongQLw+V54VtVspzWSI7Y2r5tekmYqeMELGf/9F9kET3OMkPe/d4VxsoWVaLMNwhdCovYNpOU2hkhCEuaPO2tpRmJPDybfLqwGxeox6aa4awQzVpyWXTuPU130LtjpsoleX3SNEyd5xW5tb2FhdQTLoOH5uxEIuaqdDLNwiAnnebPQeDVr7xLG9/4rCoYHIlJEGDWhW2pr0q4nyqE6d5ufmm2/GwX3k0PdF0ZXjxRMH+fBeU85Qi1jC6soVHSBPUn5UuzS3N3HkhtO4dPY8Bt06NtcuCTy68dZ7sF3bxpEjR3RSImFTWhCO60uf/zymZuYwNbuIrY1VbC29it6wh5m9J7Bn7wHVfK1dPS+NOzs3g1aTMHMH+cqsauTps2ysr6K5sy56mBrv8Yhp+kh/8ts/4H3QbCFUye8Hh9mC+lGAYyfDKhRLeeMcnbgzVP438F1CjwJivGVlnE1l8pSo97ZMgxPuGPqo9CYzgeqJN2qhGVq0CBgM+qpDI6mOtCjmzDfW1zA7M6NDaKKihF2XVP/k7TEMJCGyV1S8ywklXYgPTRvLF0/lLZQKKGSyuPGGG/Du9/4LhXWdTl0EfkPlGBV0lQ3kiwwcqnU+Kz1fmbp0GitLlzC7Z49OGZC6L2Rx9cJFXHPtdVheXkKqR422g6Tfwb6jp2RCWFBRLtuYTY0n+MKDn8P0zCIq07No19ewdO6ryoQdPH6bPPJOc0sHwHaHwPTstNLK/V4TufIMZmfmNa619avi3ak8macPq8Chi9SHf+dHRottIZf3J1HHwziT2k5mGLEhBe0ZnCreGp0kPyhUjEo/RMXAA5oDU+8Ww6Z1noaYrN7OcgSqDFNo5efQyS+g2W6g120pxqYd7zQaaDV3pKZ6ZL2y1kq4vbVfZm7aTtyzXR4ghQANP6ScEOTMzDTWV1clnG99y73Yu3efaYheG7fd9WbVk3OxL1+8LEHrdpog/6xcrSppEW1G5Cc455sTWd/awMziohaRqrY6VcXls2ex//BhrKxela/BoorlC6+iunAIczPzYHRSqfD4KFPj1C5c7AOHjomHT01QX19Gq0Ou+M2YmZ7FkjgCqyhVyRGfx/bGhnh9E9N7MDU5q8UmgsYTkzkHC3v3iU7FRj+pD3/oRxPtwniZiR21QTYQwc/zEp4ah5fa7uBLB6V6laPgVe+sFDndKGS3YwYtAxSokmBFaQ1ChoYuDZmTTU1iY7OJrfqmKE47m+tsrYB2py6An+8jt9zgyzTyaibIrhAFUW/Z8oKeN5242s46zp05o5OD5YB5XzPrMgS0egNcunwF/+67vwf33PMmdfl/5pmnMTc9qaggSn051kbdNAjPqpYvkIJUJ/GAyWpVOALHUSpTnW5gbnYaV5eXsdNo4Prrr7fvazu4/ba7jSY9wR7ljAKsCPHBBx/EqVM3YG1tXdy+2uaqophD192qg1fPnXkG2QSY2seESB61zW3UN1cxtecgZqbnVQ1y9fIl60RZLBnbKE50+JPf/qEkCgREY/VWjdEPk7syXsJ5/Sxt6/tlQqKe2+y0pNaNFAw/US96aXpvci66drtfUI4Z0SQ/F5rHJUl4vM3ygWtuxeKho3j2madw4eISVq5exZXlS3Lc1Bd1dhYnr70OxWwa1UpJMXJc3zh4ea8qoZcgN13OA3ciNYQa1w/TaPUH+PgnPoFbbrkD//7934/6zjr+/u8/gce+8iVzbPw4BjmTxKjzBfHv6E2fOHlCLBoVEKiYzzooMKTiTQnt8kU0jZWdWyR4qClRWTa7Up2wolB30D73uc/h5MnrsHR5SVU4w14T/e4A+07cjG69jo218/IbZvYfFBeP8DFbWk/M7cXePQews7OB2tam5fRlwzkHnpn72z/8aanxAOwjTKKaVk9MERVYrWidjvRSQsEWNGykcrFjjdnMsTPnbVxpWBtn7zzgxxf1ujxxqCTkSCfg+HX3n7wVB/YfRKu2jVy5irnFPejq8BlDuRhFMDR76cmnlOyQifAyXFtb4/AG6udDdxKenxDkDNLBMAfCive9412oba7ghWeexSuvvjRKDgk1pBZKLEMXzeLJsKEfEXRg3mNyakr2mKElNYyYs/W6wkzGv9RGrVYPr3vDG9SEiLmJhKnWYYJHHn3UBHYwRLtZUyODZquDI8euxfLlC+g2a3JoF/fvw8b6ppVZnz+Lyfm9mJmdx9raFW2GcnXaDnuX752oKDD18T/9Oc96xaLEQRu2IHTVY+G4+GKMyMZ46exoMQ0UiMW1isZd+dC1YrZdnYcNZ77ZeG86ZXOUATp43e2YmZlDu76NVg+45uRJk3T2YvF66VaziacfeUSTZbVc5L7HgY8mbAGt8jMqDBiZJdvsSln2SKIs4u4336MzPK5cvIiVlSVD8lhPXSAtyzo5jkwQixG8S6OlVXkd4tI0N9ZhgYJAweDPtPkkVcq5K07ge97/flxz5JhCKAI/HOcjX3kEO7UaSjyLs93E1GRF9fB0tLrNBiaKOVXDTs/PY3V1HYcPH8aV82dQnl4Qf2Dl6iWU8gVx0phfiDPAei0u9of/s+9sSyJwN5jjZd0LvARaDlks+rhaJy4rmk5sei/U293NVNbet2t0wIqfejvWEE622lmgUTZz9NQd4kqz9HRzcxu33nan6EN9LwgkiEsy4PNPPAHjjscZnS6oLm3xe9M+u2duywt2fjzbhPLnm+5+HTavXMH66gq2ttcFCAlhcx5ZtJuyyfImc+54RuPa2OWMAthjbhxyVeTC1hq9Pk6dvg33ft3XabcGBflXf/VXsb25hTvvuh0zs9PSIoRl2W2KHZwD++dYGT9rnaghU8DUzDQ2NjbF0WPju+iwVC6woH8LqU/+5S9rZ4fKDRUbReheyTc6fZ04ehh9U6XehMa98dHnojmNfm9N9ETrkZ0mxkwN63XVbvt1cLiK3kzLnLjpbhRLRXD38nD1O+96I5JhV8QH+ges/OA1n+VikxDo6dlx8zFuRsxRsVMLOOlW62VsWXK3KLQ33nU31i9dxubGGhrNbSUQQiEpDeu9xSJEDWaqJYeM/x5HJGqR3dkN4CoqRukLTc0v4r63fb2gz26jJkH8h099SpwAopTtVlPPvr29uUtXJmihA+ZSgqzvu+8+1Ld3UCiXlG2k+aht76hogI6q2Dre/Sn16b/6oGlXV8dsnRFVhoq7YWCFuFGOhu2abtsZHCQJDeEcGcgSoIqlEE2VxiEzpt9JXrTT4Omhs5uQdxvy9OO1N98tpIxNbzc2d3DrbXcDSR+dtpEWCMgQwHjpxedEpzWYNHaupSo5vjixwMa/Cxrp++iE3DcTdPr1r8fy+fOqH6cTx6DTHDM7mUDM20gWceGdzCAz5R0gomOSiIuuScRC8ffaGEijmcBb3v4eVXU0t9Z03ccefxy1Rt2Yq85eVX23OkuRjGnnoZHvTu4AfQGdlUrT0TUYuNu2UwtOnDgpp3Bxcd5qyD71l7+h0Mt2HA8xsSZpRKFMPXtxwKhPib1P6tDroQlUkJkSXXCDdWEPz2YzfmqdN3qLUMwOHkvbGWx8qQGvgTH8/ckb7/TzNbjYNdxy613I8HRf2h9fbGLNr778guwcXxEh0GdQBYvzxU2VjqnwMSxAdeCevrrlDW/A0pkzKmC0fqm77bkoKrTB6tbsr3EUTjZ9LFctyFjQoh3hZEJj41AkkCvjbe94L7r1DWytXpEwPPfC83aWp1pVG8AVTXEZbYRGMg1h1SnBqOUCc/HJ3AmyhX5uNc0p/cSf/1qiRQ1P2rsKEQZUJkdlMFbgZ573bvM3O/PKbqgDUehgSQ17LjgcNnfOwlFidkgagR2FoxhdYZA5TKQv8+up03eKSUpEbWNzE7fe8Tqp0XZzZ+R4MYw69+orst100kYayk/dNQKGTdiIheI2llpD75fmsTHfcMeduHzuDJo7NU0QkS2xXvzc6+C0x7OEBov7aq60820xdGBtHGrLa7Cu24PP3jCNe97xbgyaTWxcPa/fsuecAVCR0DGuqti23lvNSpssK2lA0mudYwaaIm26r0HsXJnLB//+vxso6lAmOwT7Jhsttv4uAiJ3+lj7Z1eJRtAzMMVjldFiCK/2npzhrTOjxsEqc+axLwWHfULMKzfu+nU33+HYb1uY8Onb7lSIxpZdro+lwi6cPydIlU6aqVNbHMX10VB+jEQYioQecoSOAfjceNedWDpzFvWdHfMxvADBivt3SUu249wshB13tW6pYkvnkshh2IVrQ/YRVTjIurIEb/7692ix15bPSdjOnLHjLWNnhjDp7G3vrhRahfehWuecGF/d2EVc7DA7ETnIdHzm47+XMDgfSv34PyfmaZF0UhzPf/RmMxa4CfHSronuAj6ZvImdOGelqqPJVAdfO+A1doEWX9CrxMkaqovsZ6f63va6N2Nnh2yMLlbX1rD/4GEcPHgE7caO4mpRfns9XL50CVubm+Kgx3LwOgQ4RlI/5liJTOiHoclPdDVObXP9LTdj+dJlMWnIXo0+M+HHBIEhTvIbuWxxGq6r6NGCeZM+Cz0t2WSwM88USeMt73gPeu021pfOCjc4f+6MLbZ7/+FjKKtHAfFW3LbBDGJVqYo2kB9O5+FmNCaK45hTn/rb31EMUSyzH7j5nYb5+jmY0TpSYZLtCd5InQ7Ey7JSHCMKGL2YixkQbOw07QS/VrAzQ3p1Yg6rJxw2NcnN4vSdr8fm5roQI+5sxuF33/1GtOm5wjQQr7G8dEU7W2fZOu891DMfSrsjcHkXKIVSLqD8W4BJR05cg621DaytXFFPEiFRHFsY9TFnVnVZrloDHYxdZ6cGBbRsjeN3Y347S6SHDO5953vEe1+7fEaLfe7Mq4rVJf5+T/lI1ppAOL11d6TZMc0YZA3RrLxvfKzVa6KRz/7D7wsuDXqNUYqNVmyOWCBj9tCjzkTqG8qdGylOs7k6scZzmrb7DR5VViv8Al8AMUIlheYV6+jBqCbVzn4TVtdW1FNlbXUV3d4Q97zlbei22KbROvJz0VZXVnHl8mVRbCOc0iLpQBpXoe4oUXeF+jaBsNEJ8k2l0Wy38cd/9Ee4++7bsY+JDR8bif969miU4/6KnWoQjFwzcdG3xZJAMbN+JFMQHYnLI4Ove8f7MOh2sXLpqxLKC+fOGiHSVf04UBU5i5G/4AUOfA+F3tg2u5z34BGYtkwj9bl//OPXhF6jvp8uwRZnGjFg1NGXUpqN8yzNSVMxgSNmYZ/ouQZyZuc8ewStE+fNhpla2z1wLVpPJEkGt73uDeKNE3VaW1tDu9XHvfe9HT0S6nqsDrHFXt/YwJWLl1R/TafFMl9GJjTeuFdwqurFgJAwLyNAiAxTb8BnThaBlK44dYahu332tG8cZ2k70M/T8uOVAjnUCX0yJxae2nvjUBrqoQze+Pb3Ydjt4erFl2VzL104PypTskNndzsvhUmKbBvVeFCYAwCIsNds9Wtp0akHPv3HCZvEcbEikRF2wj5odjeAjlGHP8XGpto5SOFkyrCYBiDqFUcbSfKVMTMzoZN6vM5bu+s1xQnWYJZlwjfedieuXFkSAZF9vtge+g1vfosQNMba8fCbW1u4dO78qLOhjd+gzXhZZskmWlThcC69gI4cPOLyjCgsRy0RN36dkn3m8UYyJeLqEOZY9N1FlTfgHrlpDyvCsMZ4pC7TQXvj13Nn97B66ava0ctXlrxvmrFr4npxX9G8YiMyeRKaw9GeCNMsNIOyfqbKE6Q+88n/mZi63T2OgWzQkPgIAeiI6Wxt503HJNruND0tD9CPNLJF9ERJADY6dshaPlscGWrcvGe1+VANOFROdN0Nt+DKlcsiGjJe5K3uuvtNKp9ts10jGZnDIXY2t7C0tKTF3t0NnJTdHSV17tWRHKfxvmynh1Dy93TqZA+9twq/l9fL8NLHGyf0CGuIvqD+jCYg9j9UXYAsdhSym0hWtaQzeP1b3y2zd/XCS3LKrl694nQwW2gzpbsHxIiE4EWAHOO42tZ9RjlFrzVztFBj/cw//BFnWotkDEmLcUOiaHPU6DVtao7F+uqsMmYDxxeetczRRYg2kLHsru0O6lOoNNMXcRC7YlI/gJ1O2613vh6XLp5XcbmOccxkcdfdb7Z+afXaCPAgAHLxwsXRafajSXK0xjQNPK7AAAAgAElEQVSvh0puasxb9zg7doUgVMMR5Pw4SCP8OfBvPytr5MCS+KB22t5wncczSSgClTQCR+z8kXBwsQG84b73Soiunrf4+tKli6MTl0zQrKCB9xcnnKiemxRGH6G2Y6FDsEJj8hoSCP578B8/nNhxjP7gzh6hNx8XEgDiKpHzF2dHMakfGoEDVmd890AD4YrEF+fT4j+2prSzSEjmkzepigqj5cSk5PMl3HT6Nly8eAbNWl0IGXfg9TfdgcpkVa24wtPk37mzFYo4C3bX8x1pcn0TDiHVdnw+nMj4uxweXyA70NVACk+YasxU9zIjDIc8XtdZ2wolY0fSNHT8aAr7tKAdJX2ETeL1971P110+94IW++LF82aHw79RGOzZRvWIsYPkLTHz2ub7Sj2PHEKzmnHagFDSz//TR/ycdPPiVJ3IAckxsA5CmhTufH719GE81CiTNLbIeix3vJi14e6WpvAMWZgIo0BZmYyFDLsxOG32DTedxoWLBDi27RhmAi8Ts7jpphuxvbkyMjU8Punc2bPujVvYGBy0sFcGUY6Lnjkv2oVj7SflTwgxtL9FoY5Br6aZI4YOkmOobd4rMoYyYd7VP7xyhXBuhzWSYYJjN9yJ+YUFLJ99XkJx6dIFT8zsEkkS1xaMDKKq1Ha9JX9Cc4+bFX3v8xtRTurBf/qI5mA8WcBBy5UXROdsEpEIqZbd4Pvp8qPdYS6It0o2BIfgCr/GGV0kPASiEzF2TJCpmzghwHb88eMnFFY98MBnMD8zrf7m7V4a3/QvvxU7G1clkRScdqOJJ554VIsklE/OmSNebqujowHllTnvXZ/EBCBsXxAwKBzWsM6OUQqKFT+vfi2+ix3NlyCrSCKQNkcIzY8wGrOcRO+faioshfmD1+DosWuwfJYdKmpYY6gpLWKJFUszO1FEWDjPzbYiC/V1k7Aa0STmdmS7vcFQYA2pLz34vxJzauyhTUpt0qRu2GBdyQlzZlQ3xPeN8dQIpqhk1h0fE9rd3t4SHnVGcI/WVVnYwlDdcX/aTd6/1ezgwsWLytpkSK0Z9lBvDfHP3vcvtLPpuHCR2IjvySfI8DAVqSOYvSWnhMpNk7xgn6jY/fKmvdWlhWzWuzvUfbBrHdUd/T52EcMqdV3gSSd8U2g+PxMkujSquTZbcuq4rOixDmTKU7iLIea5M1psljqNvH47RNPGz8+Lym3FDPaKGF5++2ixw2FmOXAwSCTsX37of8lmW7Yodl4U5zP+cFBE9un/a+vanuuurvM+siXLsrk4zTMdGAghJc0Y22BjoLSZ5rl56kuf+tfkodP/oy+ZydBppkmAkkkoNrbBKdB2aOMB27JsS7Isy/iiy+l8t73XUdEM2JaOfpe9117Xb31LXYzxtLvTwR4pSR9LgEZeVpvIk5QJtIYnSxJVoAiPCgRAGTpVePBnQizc79H2pJ1+/e32zb11xtpsf3n8qF358ss+WSdIVpLteGFyvWrBs9Gx1QzLEJWYoCejJ1QnF0gDa19LpQHqjKhFJoxQa288TyHYI0pGTcI0abtzi+3Ea6+3m1f+pz14uNlu375pG68hOVhPcdqonJo1wXvt0kGTyQ1zlMRifHEtAgP/+MN3kgrhZuGHkB580V4nVu2D1nSxWD8qy8zI1O53tZh/opU2C0nPO2AFfxbJfKjG/Sc8JkA8prHvc+2Vk2dZDHn0OM342+3alSs97MgIKJ7ylAvLCU6uoJuqMgVQalnjmkZYpU2W5jGO3oyI1GY9RamedAnPKBgBlgQAYrQBrquDMNd2JofaqTNvtLWrVwiWYHrYqNVoGBZhzHmukM5OngfohMUh19f+qCAUT57ZynO/+wWRKnFociFCiJ3qRFYLtyAQwOq8k7LtG8fESlBX4QYt2u6nt5kSywXWwpBxCKrTIAeeOEnQjG1VgmeunX7zr1gQQC8TrgPM981ry4ImdfuVCYBKZgw5hC0WsIGLY3oLLbBKrqlmqZ/NiFW/p+RTAh5SWaP6ugaqmwpsu/7tqlfSpTxYmKh+qJ149S0WQkDTvbGx3hEv40gNkASzcp6AoEepYazVuvMe3XYnawc1HrTJCFdU4406pdfZbbRjYdNAUkpt63Pao0T4kvbMueIGFqpBXYstG2SmJicpFFZgrPAAMOq99FyvvfmXpKcAVQe5UnYet6t/RNVoh/9WGFeRMlrsLB7Xx+YJz8AowA9dVTun7iH37Rx6pgNFjQOmS7gV/BHWA3TiVD8Y3j7u1zeIc7vAMgVth3U92E6++jaZHzfvrfNkax9k4uJYZk1xVX6vqGrlPGBf5LDFXPR7JtV7/sN/0TmK+q07ZueAC+1eLv1dthsnAMNJ1K9tUJ5TlXJsaj6nPJ3Zi4C9Vi+YHERsR8hnnLB3rK/TFOfxe6Cu/s53ScRD4va97bb89dV27x7w5KMql7q2RiaBv7Q8g/8aAVdoOODFiU6kqFyT90LSJynwJPoeJUfOjeiD2uwxO2Wp0Y3yReDRo8x55s2ftDsr19rdzVX2d3HsYuaTs4xc0rV9/Sv2L1UwPKfEQLG6BtoEmzf5+KNfWhvY1ibD5FOZE231L3XI/8+Rfjqgh8R0OhlyukAGD3uM6TScqxVbvSdmhJKnV8HERQeGPSyJJvGhaBfCxbz1wlI7eeo1MiHTmWq7beXqdQLzMk1eWkm7O4odKXJhBomotjnAVKatV+jkUIVpSAyPFMbAjqzNkkJNbE2CeY+TyGQAMjoZuqy5W/DEVeAgwufAQjvz5l+3zdvLbXVtpd0Bu7OdUzw7ng8jq6kNSvGoh4LVfyrIWWpVb3YO8uTiuV8RSox4MN7zrPxLavIL6c5E7hoLMsKA2d9KzMffcy4XQkfaSrSpGqCYe8bOzXrII3VL5KYF6e79x+3tH/+EuC1K8nSPNB5Qgdg2fTYmQCpdXrQ96V6lEkVHHDloCWgBYMz43LGHnPGl9ClOTNS3snWKh5FnZ77dzh7Sy2Ql3tPAG8wCwbVFSARPQA4UNvPlk2fb1vptjuVYX7vFe0k51CaMsgeZQNBDMK19F+p9Cgx97TzhF8//2o19Q8fFfZcS1qnqm20Ok3SI7BcQCcDYJHrDO2itfaiGOzaGuz2ocJbgaSAAsy+pxj1+z2kSXH9j61F78y9+3DZuL8s32ttt6+vrbR1jLayZ9LzJHThvwFh40Fv2iCK8KHZ8sAEsBvnm2EBQhuTa+X719mkryc6gUcbpfcv6wCuI40n8gEGIWOOXT73RtlZvtdXby+3uxpr6203Bid8H71miADwLINQcBxFHLQ0Y2WQntKANuHbOo0w+Pvcr48a1oYq2ZSP6ifZb4nvzC0JW5gTq1CTcGDavxsg4DVBlcsaCWvUm2rusmiD935BUeLOS2O5Cte2duXbi1TNtA6dgD1TVjQD61bVbXaYZYbg2YQnqJ7UKKN5JVJcgBhCsadaxlKgpdBTIQYKZcq4SStKOEh/6AbbjIBzQ9TAZQAT5aYHSlaft+6+cbvfvrLW1G1fbPYApe11cCS4Wh+y0Yj16+jNxvN86BzJ/ZjGgzum/fPrJ+/TGe87XKiRqNb8QFYV226ouqtrdpz1mBCI2T+p1oCFHBDAECCafaUerUiRzmFjh3E7QcB1qr5w63TbXV0lnhc1GVeyOwxY9B3qzTBvhWLg/X46odsZwXyWElFoc5EGs1ZcCDXVdSrbOlxPznjCOZV4lQsgOYZydfADhzxi5USUJRPjD195o32zcabevf9XubK5zs3ELMkfVAbR+NojIE08cJeKOJU+/x7etP01BiAAvXvgNN5ujkKIyi0cH0Bq+hG5UjRpf8H2wAbFR+3PN/Ey3s2Mel2J6PVbCL17fTkw2qsezOiszNeLJ3lw7ceYNOmRomwEVFurda+urM2FXMnYUqHjLAe7vW5nkxvPtekq0L9Ze7DEDoTxoLsBtLt61aB8mobxW1G5GfDLxEu44ok1R25cX/4MfneD1bl77st0hnQgcOCFMD3pONvYmpLYH5kWwHy2SZ0a/WOJ/ijsPixIstNkXzv96mrSe0p0eG8GN1WXYQOAZzIEWIc/dL+i71RM/CgujlDjgsb6uM3bJPwe5mQpVct2Kaw2AJHFKa6+cPkuqRoyMPAjH78GDtrJyvTtMqqPbZsXw+zlzOpMAyp8Jl7KIPZal0+I0qHMC1BzklgFJkNPNwIQDaMdcuzppoImY2vSJls4ZAEccoOdefJk+wvWv/ov1akQ2nLyEWjbsL4afu0NEiS3BrWhanOaWMI5iiEJJ5eO7N/7Jxfd6R8jMD913NfqmZgvwcLoYI6ePiDnzCnbDyRWqcn96tGqB5Md1kmvHpU5zCHPTXMeOyvmF9uLLJ4hU2drc4MlGFm7l5o2OF0tdW0I3SADY2xVOb6NjcjK6SQkg0smLaAVqtzQxWoDU8eFChVU5N3TG+ZTDJg2pJoqOI2tz7cixYxza9tX//ne7ufw1JxbSbNmHSpIIDpmG2TSSDsATUIg6Uqj0j+LQGrZMDBCe8dNL70+hluSAqBdbR9Y+kRMgWNioA0gKOwVdyYEdQsNfWlajgns4ZUjTQFoWtegFzKbIRimRoahN4Q2+xEwoTTO/+FT7/kvfaxvra+yUQBsQ+LWHRrFtdMIoaVTxgkeQMJoYU4+GY1nbd6qmx6IKqKiig/B64z26AHf1OTQaPoj2KHGrylZn+Pt0Z9ouf/FF+5uf/rTduHalXfz9b9t3jj3J+QfJjDG9y5aoxmgGIEgWeTxsjvjBRDhss7b/Yx9BDt+0Tf5w+QPS1ygLlLgl+12a9N0JghoqnAJwimUze2xpG8GUnoefiUZaeCxtYkIi60Z6uqlj25O1vOm6Dv8ywdaFvftb2+21s2fb2q3raqnZ2WnLN67xwYW8CdiwJhZ1/yAyldQaoEQKMdWkCzelb6tv/AgKVE0y5EfCaEfSCy7BVP9XNXFxqOqTra7ebh988G/t5PGX2xLYEiDkOLEGIdAEGlARcGgQrorHkdUDH5oig9Tgtd6mOMPJ5oPkQlalLKCzJQeDxlE8iJ2NLRinI7ZbiyeV5nRy/xMbqhYVLXYqO/SwS3IAzxLkClUZF1D57uScITo725N2/NSr7fbNa4T34HpQ4xAOaJioZIQq1AxpKS7v5yBToQz5VTCkVJuTtJqyqCqQpA5dHUuxUth/KSldLHFKwqoejnC2JksYpcB32d0207JnDXAtlQxi+AZ1jfEW2zucQwZoFt6LnSPBCYDwxxXL6lDOL5joCKFXjZmT1sTi4SEB36WtsXTizxj8bEZ+P6FSTz06hNCNh6qUDRd0SDEkXtQUlS6Q8HeceZMwZdYXBEA/Ovn6W+3m8lVgSLlRt26taHE8CObbMoI5BTFVaEmqz68WWzk2KnP63YkBB4/aYqfPBOYMX0ySlNJjDVsxIE8lysIeGJw8b6TcNZJO0n6D37xGBLTNHALPxXArspklQDO2s0NOuHtb95iKZqOCexnhXzFE+8OnH/Bk9w2HNDlbJVumJvpsthIk+jyrRQnF0ozmPHPQL0mpjkoQZosM1TnrIOhfeDC8PPovgi6hSvToIjiNsIEnz7xF/jEAnHEfqPEsdGL5qPP4EdFYET5ojapOa7go10WFGt6fm6PWpkQuNDJOzECFIudO79ydKGSz8xcFLSFpcQiUANq24zjajqMxs+manKCnjXCR/RkEufb6EYKCkpSQMnKrqYjDeWXZbJbnAhEuD8JeLmdw6oZn07PxgiHLaWHzuGdcRp0GKEBuEoP60BbcwwID6HU9WbugJ9FZwhAE6plqEz+bbz9CL9gaxkI+pucKB024OYdp6QFmbV5NinjAePhpeNMzJKmihnvNDpFGUZSQaESCykDHTfrcLJxId7pogfU93Pewiz5xDHNAcmDI6eJ5nMPZt0BZ02WdsjXSXhJysTS5X85FFDhyqk62Ptpicuniu+JUsXwn5qZnTika5bO8XCQuajwbSu1g+yhbaT0SRKUXVQkUdW0yBjX0iPAbniAFD5wGCRI3jIYKRNdcIWgP+sGfnyAPORiI8LV8Q0R1GuCq6hKEjjPLYJON6aID4znaCZ34bwq7bDcWcjbRkky6kiEJtxiuWhBjfxlaudFR3Z9qicY6UXNgpMbhxe608eCkJ67jzmd5YeL8cfMOmDQXc1p69+hen9pbBQN/R6jKwfCXPv5N3qKoKpXWuHnGnOUEx7mQsyUvOw5RVB3SfLAb8sQ1mTYmS6xC4u5OD1QnZvP1gv4Erhz8pVWNcnQkVOP0QHvm+Re4qWBTwtfNWyukn6A3ySxWAAvyVtP7VHFawZlhpHIydTpxo5iT5E5MQ9VG4CvXe48qm0yiT5WRPemw7KwUtuOBQDEK4LFOAqn4OEVtx9xWf6mPniZ0GcIoAYxGpq2HULDEabWU2LFWpTicmV8KnZhata2m09BbXUZlDJ/FaKI0ApL7k4wOJTwxL3naUxcwjQf5ZJ9u3BEErBpBLCRIQiqGRm2+PfEn323PPvccqSTxhRInrscMAMD729tkG8LG0dPmu3gRDaiP/dVwtREbd3SttRP+LSEbBQ8+OzabuYKR/lVUEpNh6k5DruCvJFNY07Cxw0Go5ARjU+P9x//JhufgAcwoBy5Jd534oZm0T5MLH/0rq1483oVdIBs/c+xl2fqm8WYHNMwktQWcZHCNcpSEpYs5Yo5zkMqW4GhhUapDe5EqOQbtO5QJCyEhSsjWOXTDS2AMIRrjTp89S55OfA+c33BQOILJbI1KWcqRxL2hbSKgSiIp0zcSOXIKs8AAEEbFwjT1EK33sMthGrWV8W69JOq05nAexeeuTXOiaF9KF9eMNoWwc/18GPJs+TlOblXz6XaJj9A10acX3p0KYTEQFUmu0AmxPY8nrGFPQwTojZY4mZOBZtKecnIY6/qUZL7IiKPtnTvMgfCgiiU7rWIB1ZDVssp9ILcDWO9UW13RlN6Nu6tkEEJ2j+zDYPhzxSxISy2iMk4anrrN7s2kN9PrhQWiEBotk/KmzMFgYooDV52umLeo/ZiebDYrab16WMD9xdPucbK/V0NevAM2P/kJYO/w/ELhylzVCCsagDabF+bpHl2JSONFv4v1aFRRdDId4xkpCjyV0psD6Ie/0zFQykhT64o9g4MWPDeegW4ZhrK5vpzSphZ+FDUEPFTv2Cuvnmkr167y5e5uronczYkdqjE3K8ZZVNyMcBJOHGrSek+ke/GFgkpMC+7BU4TnOuAikWktYeOl9r35hjhp2BycOxs/x+3MetnJ1MFBfludKTBP7Et3eKf9MG0XES0DRcRN5vQDHM5RtIr2JC22U8JB4cSBnpz78JeKswtTLz3yvZEZktrTw0hy8AAOLQy3ibSl8Wx42cp88TTCMwTkx4uEFRmqBpkSXR+4NQmF79VhROJbSYQA7rXjp063G1e/5qJt3d8gYgVCxdKsNUV6oiPhym0btEBEKhZdqBipSxHQJ2rgOAr3VGX+p5Aoo3Ajpw68brovpBFrgPdmehmzxgszFKpcMS34LBNYKSfjul1/SqBSWuY77Gl2N67fSXNc3NFUxZiWcXhpsy9+/B6LnWH94xksqqOnMp33jqOGFB4+BqaeWdugGVgKbVBnvt+WOO9aJzfM/iwPTveYhMClU8+G972I4kSHEkNbiJlQEjq0x/bOtJ0+c7bdurHMzQH98vr6Gm12TwyRqQnZJRHEQjUne8dqUkh7Jgca5lknjGKumc6oHDe0KjOGR1vSA00TTn93PO+0HkOYMVtLGyikqPyA0e0Slatr6oTCvMmpVVwvhKlgVPiKiYRgwy/Suks4a7TUEy5WL9xoCEnd7NjQ/FCGXW4lZAWSGbUGT5eDUuz49MDeN8DpTBtwVEzKopmDOUhwR4GCqp+w370+sD2AgIAIEepx8+cW2osv/Vm7uyZ2QHCRX7++zDHInNG5s026aPGaisRWeX45atgcYsvIqCBHM0PQsanyDVwx8nShhGVDaOVgIfqginU+H825+uwBhoP4PLBkAQlkrSEQ2fCUhKN2c/BynWQy8X1om5rBjOfdVbYrez22Z+jFk63TkpvGkajA9rSuYlIffh7JlIqEIKiYEs8RN+8xcWcDVp4Ym4CXxwMDyYm5GrhGkitwsLiAbmLTiXHNuKMolZR55pnnid7cxcjG7Yft9q1bYmBIWLgLFWlqjU5eo9HJQXsQLmQikRAJcBNcIOEkQA+HBSgCwgh4b4bajd5ybW6yWlgLCCiETHkJYMWlIdI8iaQLGvmjqnFtrgNO9UzBTodOZkbTCuTfKIGEZ4BpwM+zrvHQuwBks2OL8+ewJw6H7IFCF3Ni3WGoZn2JamR4h5HIJF6wcHHgEo7lMwT68T/E0wovSKVpcLwkVlkraJP8nDXi6bQdXnq6PX3saRK9ovEdDhoHssGjNEpDmkWxKE6HpuSJ7opwXla0RPADqUtrUJxJOnT22IMQSVO9FlKsSAk3Ewfn5NHj3xZB3UxBCNqyF5ZS6gUEWQPl2CJtxAvuo9hfMXRYDpPLx/tRU1mYoE0gBKHepM934fy7PY5KPJYTJifdRZJCCSkPO2KnP6v6CF1HBCcaItAibeDwvOvvihpT6UyoRhVCNB4i92WSBO2rjx+3g4eOtGf/9Fm2Au3ubLfVdbQEyfFDEoV14eku2RHiiCoxInADrquKuatXCBMJbHQPd6g4IVydiK5kt6zm5YXvtsXDmlVK/8CtuVgH2VRdm3l+1w5U+VPuQRnFsZZsP8JweAsl1gyjkbG+bFAwVGvUuZXNSddJNDQTM0hqZbOTcYlKr3ajH+GGmRaa5BrpRYkwdk1ORkhsArcdUJ44cvlcEgVJFQZUgJ9jQznv2qMaBpOCFTrGP8LxObjQXnjuhba6uiLmgqt/5IJT4OLFp5l9H/BwRssYANE99vCrOvkD3nD9TJtBzWGzpbDQwm+kT0LKqNfkGhA2xbGSI6vWXmUItykETASlrm6wJwWyx+HGFITN2Y2QMHS91h60ivMkPGBffPbvU0gWbqzyn9R0Xjqbig2A5xwg/0gc2GlzrjdqpSaEEuPGS8y196dgByugVGPgSLGjSSRQLbtmjVLn8eMnCDaEqn3n5//UfvjS8/LaCb5YEG2XB7+HmUGU13a+vE9Y8NFtOcq+FE6nP4n/DkOzt5hajuXLAtLs3RwqCPW0rFOyma3dq2k6QqpVu7ukE81mMJo1BIkPWKNSviH7ldw6NWlICwsMmg5aJDXNbPhw3H1me6aN9ihtMREAOQAmijfAQGHUKEAkNSoEptCQ+BPCFQdCp1d4ctko3XMmGgj0Ju01ZleEnf/nd95pZ86cbv/4Dz9rf/93f9sWD8+3xUOLnB8GbxueNuNSsCog/jVlCEMbb3TQKR0IWPq7uA1u8Y0GDL02n7Hi0p0jTZMFO1fpvLoNyZzobAVWQbiXJ5N3p6oHHYjbh2nWDJcCQzPeGeu4uLRkLZsSrBy43vi/73RPLl14b1pZimJ/ZZMVf2MjOLBlH8mNPlP6hVPJ8bG+u3G3PfX0U7LplHrFhUlyKMQTLzgkP6paDs8YDRmTEuHA1VSSVC/1Y87sRBPhw3ZwihLnNz7JiIkftKUlTNgB7xlCL/V7YeKuSAKM9nSbrwo26ekOl5uydez88OmjlvJ7xjbG58m/eZ0219bW1zgkhtqFhRiphK6u4/OUHEc1p3aKmJRK0Yoh3aNHjCggvNG0iumFQuUhKpypk0sX3p9ubm4yoTCcrlrBksUeIL0JHSV41wn6ZcNjmwPzGaBD2ShVYSCRrF512g6hNdNWo8+FL3WEY0m8xF/garFeiGQDxiIjiy3BTCZqfjIhXgsoEKxv4lRQXfPkmesFz/fNN1vMpYcbpfssLKjITmcqQA6CwBpKM6eDJQjcVEa6s1vmqGSjKRRutpDGEeZOTJFpNRoeU54pthtTgZL8GTBuJ19szyM0vBc2OxL57U6ZbiZ77hFNpeEbkqVwJCeieucSfgLj+u8rohWFpuJu5ZI9ycBCoSyXwQ8u0EcYR5Sga89hlBHnj+gLagxOk3LvimnxBRN3//5WO3xoUaB7xPHz8+3QPOLgbaVQd7XoOAAYldSnHIw17/6M1kOFHsKDwEQcjHotItG+ptgj4j/AhHDqMMeD/kkn1TPmb6YWoG5PxuNYN8dPoAUPlmCsDZ5JPDShCoFJo4N2+ZPf9s3GpmdTojKrg5bNrp57PNrYOth2Zc6GdqAtBidocN8Zv5S5GS44xGEj1bJDF9zTfaSdB1Q+geJ7OVomk7U9xKhGxZdqm03SvWYI8bzppWIee6IRj/MW3m67HSaBxTDpzhyO8RwqicYBlUPmvHRYD0ImaEh2h3V11gph/ygwKI6Y3A4nPp8VocCgueRmylPrzA7adIV9cFjjNPJk/8fl302JPCzzr5SEGHTGRajlWboPORs9q/5lnxlzLqonKaceJy1pPZ40Oyg1BOLfozatQUgQU8hsc7+Mn8pmRwPd37rfjhw9qkEpHuGgbNkA62Xj6Yi6GY+x+67CIWwe1b5LuECSJgYGGPLOnY127Nix/2f6IgjQz2n4i9qWdhnVO4aedvwQdiE7FzPFOFzODu8xYGI2qRMBMzmG8cA8w9T8Lip5iXhkFg4wvp98eumDGXxCbHNOeAXwRwhy2hmse2J8atjZCHnYvU6mGZmeZ8Eih73zOEP99+yJ8h7FAcLCQ+UlYpAfIMHqwuZ5liNe1/35Lv4c1X3meblJT8+g08HMFNbYyBPlx3MPwZ8hCIFSJSunRFBoJvX5/VqxC2k89jIlKbZ1HAZBmxSDay112jXgHZ+7t7nJwg5VPFuD9sQV68YFnHx8v5c6ocbjIWsBRzEdL5qXIpDPbSfDSYqNnG2pqfYDf8c1qhbQQBi03oxMnDzYQTyjQHH4CBRyjDGiFtImI5SS1BvAaK4xLBJ6v2BSxvuMal7i+TwTFjNdILDdMDlhJkz7boQ6WMpJKI8AAAdhSURBVHeFTPM9/Rqn7SGm2TLZokWOZ87nJ3wJFTxtWl2TCMY4SHD8nO9wf7g6QhVbU70/gokKBbj8VZk1NxaWfAk1xOXLv5/SPhtaEw6x2G+l8gZTQiQvdrtWYvAgyYpF3UeAcpry0hEYwXoH9kzJj9mxilGfta0X8SbOrainFL5xRkhaVL0IQbf0Re8/l6DqkMlOjAVPn5g1aY+5NQmIGss4M5qJEPO5g0MaT8UTrB9ULNYFEUzleckzVXufE571iTnVeqpfLHYYzI442VwXLazv6VYuv2tMwOSzzz7iZsvDEyYq3mtuPLJiY6pMNjvqvnrrWqJxklIQiGpXCJbWnrGxuSayXimPytFTokYxcwowOfXwgBH/Aq9u4rze751JQGFuHAmfoDxiampdOUmdYQORFxdiFT8TJaZBfGFWNudKjbBy7RD+5tBwhBRNgRJSWQtBqPT90cwY7nIsqPP5ps0A4RBKuHpOTQfsozhKQ2OHlGGz8eHqqWbzUz8epzykqFC5QY1kY7Upo+gxWoaG/R/9xFGvtQ5bncR45ji5meKjk5ci/igYxPGSWgRXqVOdTswM4cvfIoiBGAffpsORcIr3Mxl+/02364hFQdGLBFuqM4DGrBlMFd5V5rACE3WvmkmMd5/3UM1cdfZ68GifbVblAMuRC0NEogL+jgs+9Ds+//xc51SpH0p5MKiObE6kKDndqp5rPbyq8bHE+lskOLadoUahg8qmj2sPxCfGIIhZUClQePxaCBPjwvbbYQmNNq6TGrJSkE7d+lQmWRLnbzhW0tUiBxi5+pz4qn6x2XHWlMMPBNgJmd4TDm4ZIV5qwTo2/969LQpGZ2xy/h73TBkzZgIags7XnCpd1T/oG02NZ8QrNjtSk1NWN50pOvdJMzXKAWUhtk0hAY1pGBAumqmqKbJww2kbZdMqEJHq2PiYAZkQJVeGV6xTgRQu0SX2/BGC4GVUsx5hTH+GjGvEe6BZgfPHFCb2cMvJnzwP/qQ69vgFePO5djZoqOtBWJDTCUEJiie16W9zziJAua+c2j2GeEAE6T2Vas7BgBMatNDsgTKYz45sYvfJF1+cFw9anddRSlYjoaHm+AhGbJaVeMc/V6ejhh9V6rT4aQ0a6jhCNpw6lDrdb+wifjYuzxsBVSZPSQdWoAwqYJxpZ4mkcalU5cSYKuvBw4fUEuRutIOVEI4LzchE+Paoea/GjI8Th2q/TzLUveJkkcQP9RxBzmZn8/P9CBQg1keOLLloFKbkUaHTvjjTZh5Xric88//8XDZbLrw+GDWkgsUgcmNhxMWOvExV9yqciAqK0GSX2YT+UP6bed2OIEHixm1GrhvHo8c1hkerNtZasKnhHTZDi2xwIBGv0DI6BQinDh9eGsCA7n8Hj65wCM+IpEo2O2iQnETew5oDahYLOBoAM21wIGarxqwaLhmxmouoMbjWAKp+ND5mPaJpIgSgBHvyyaOMtSHJ/YAZCxw7zh1WnA0vT433mT2ZBIqw0XoBVprc+hNtkOZb/Vt56H5Dj3msKoZ22JmsEepI3qr5iGceCR8/F2xoVqWbu6yGHkUooRJRi0fOLoBJBR8WPlflWBErPK54huQa8g7yA8yYmNGI1hJxxMhs6CRLTqScqoH/jg+E90h0UgWY4bCLRtV5zufzp1S6+VFNeAAPPbTfSSbxmZFBq55xJEc4LcGH5GVrI0EAQ8fEpzbSmbId1zDcV2bQtVfWwQL5d+gngCiJk7V/w7UnmQ44xk50zeLwUvH0MDNYhEMkiEOodJA0mouHl8hJokze6GGTf+DZIrPGr2cBq9kQkFBCzejezmWEPJue39H1k6cfEYUEwKEVhxBopHUEJEIg1a4GSp1wMSly0KyjBX7fh4BTfQEgdXMh9hICMJMujWRp4VVPjuufF+nqPjXYzgIgz5WntcTY+G74TmP0qTWcqWMt24akdk7GpkvCR9twTnwWJPY/mw2nJeqf82bNTMgcOMuhYBnU6GcszsEF0UzVzc6192ukaBeZORMRWJtFSCMEw2fQy+XfEhTXsn0N2nN7/DtZF/8shy+Ck/tqr9CSrGIINS8STNCsPjwo+vJQhEwAanxspLzrYMJif+Nc4PuCz6rmTKkMrpr5ZJUsuTlWCTOJd6vW1H5xX5QZM1YqKjtOVcITLeAgxgkvSxy54cmbiNbsDTwnlPgQ9nlSoPlX8axy2NCgGF6xkf2iBpvF8/YTHRUPXtCcQDx3nLrYeTbulRFMSHAwDGQXrUqwOKXEoO3stKWjRzsQQSHfWMH8HUxK7D1zFm/A39y9KenyaGlV3Kmlocbria6OQiS7OkuxPbKD8F71QJ1+0r9E25yGP6u8uvFU/24zDYlrdVjiE6g47+S+a+PDdAxgdU5U7CliWXB2Yqgc4LoLwHujros6d6V4dmGB7feO1SNssPOY5Y2vsXnjpPJeU+H3EhYpATL4YhB/R4j7oeImSVvBK4eNX1wQ5psACg+hjQboPlCiJm72nAbYl0oe7TS+7/73fRjI9n85OQ8T7wFtAwAAAABJRU5ErkJggg==">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -869,7 +938,13 @@
     <xdr:ext cx="304800" cy="304800"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="22" name="AutoShape 14" descr="data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAHsAAACkCAYAAAC3r1GFAAAgAElEQVR4Xmy9B5Sl2VUe+t0c6t7KVZ3TdPfM9ISePIqDRhqhZAn8DMu8hXnPmGXAawHCZDDmwUMYk0GABcY2wQSBSBaSQBKDNJpRGk3OQTOdu7q6ctXN8X/r+/bet+7o+fbqVene/z//Ofvs8O1v75P6ylfuTwaDATKZHDKZDIbDIdLpNHK5HJIkQSqVQqFQ0Fe++Du+n7/j116vh1KppM91u11kUmn0ul1ks1lUqlV0Ox19bjAcYjgcAAkwTPi9XYfXKxaLun7cm+/n/XuDvq7fbbfR6/X1Pl4jneZYEiCd1ec5Xv7ni9eIMfIavC7vw1fcg99zrNlMBvVaDYP+ABOVCjqdDiYnJ7G+vo7+cICpqSmUy2Vdj/95bSRpNJoN/Y3XHQx6+prLZFGv11CpVHQvpNN6P+eB9+X99Cz+lXPG8fErr93v9/X+mAP+rt1u6/7xe36en4n38JHHfx4MbL1qtZq+JgO7ZjabQbFYQurRRz+TJACyvtgcDC/A/5zAmKj4ykXW4g046fZ3CklMLNcAyVDvyWSymkDekO/JZCgIPc46uFx68H6fP6JSqaLZbCCTztjkcuFgg09RQAYDDJNE10mlbHIyubx+jjHwPrwff8eJiYnm2PL5/GjSY3K5yFxwjovCx89SkPj+drercU9MTIwm2+YgrbEUikXdo9Np6bq9Dt8/0PizuSz6w+FIiDlPMU6TBKDVauna/Bs/z+cZF8zYWHr+VErvp4A1Gg1sbW3pd5VK2TadhDBBqWRj5TU5tkzKNif/a30eeeSzCW9EqaBUhzRmMiaNsWt5gZAwDoSf4QXGX3wgTjDfpwE2GppkLn08kIQ+AbLSHKYN4sFarbYmm/fkq8MBZzJoN1vo8/tsVg+RzmYwMzOja8YYOAl8qPHdHRPJa8Ru5vslKJkMEkp9xrQDBW44sPFo0pEaCXOz0USn28G+ffuktXRPLnCvp89QSMoTpp14T16f8xC7lb/jz3x/aAj+HEKgsQ+GWshWp439+/ePtGyMnfcZ9Hsab284sE3A3ZskyOZMI+dzuxsxFlnP0uuaUHGxbQdkkMvGg6eQplhwx2ezI9XDwYeKp3qhpPPv8Qq1rxtQLfUHSHH3+04P6YWEwXYIP8Ndwr/x//b2ttTOxEQF2byZEk5Es9mUFOt+aVPNMRG8X71eH/0cE8txUfXHK8yGFjpJkKdK5GK128hkM0hzTLwfhaBQ1L34GalvQIuhuTIjos/SJHXaHZTKBY2fgspdSIEYN4tUrRT8MIn8Wwidmb8U2u0OUukU8oXCyByFidI4+n3kc3kMYLs1TClNCe/ZbpugmrkbjjZNMZ8zIX7mmYcT7hqqU74K+bzZwIxJTbw4UP6ev6OEUgVJsoecexOOUCGyYbk8qKz5no3NdQ2CExFmQjug29X1ymWqnwES3xm0vnpwV/cxCqp1jqPX7vBxkc3nJQSctGq1OhrruI2L3c3J54Rwgig81CBSdy5wOZoPJBgkplI5YVxYCdtwiKYvYJg3PsfOzo7uqUV0/6DdbWsecrmChIjCzvmlLdd8pmyhzBylpJK5cfjM3ADtTlv+QzzDxsbGSHiq5Qn9jf7EuGngfIdW4XxwLkJ1x9+kbb/ylQeSMp0E38X8pe1YU9vhjPHBeSHZJ19sk54JORJUg8WiSbfZNu6+oSai26V6tuuFitNuGZrTw50sByudNtua0KY1sb21je2dHZSKRRw6dAirG+taBNpH2ihKeKjDuG44llxYTmjsjBi33i/NQ7tb0PWnJie1O+kzFMsVrK+tI1/IY35+fuRvxFyMa69mo4Ecn6/T0Rj17IlNfKfTs53X72sjcY6pwQqFnNQ+BWVlZUXjp/ks5vJaAy4kf8c55e/54nzKbGbMNNCMhXaKv8VGDBPKcfLznA9qPdnsxx57KOGH292+VEkpbxKdSnEf8UY2aDpwox3mNjkmOLzyojsLcsiovodDPSQH1u31sLW5qZv2B2aLudgUECrJGKQW39XpoD+UWjOv1zx/Si2FiLuF+jSdzqDb77k3PpQnigGwuGcR9Tq95kk5W/Ja+wOZjjTv7d5uJksHic5kHu1WC8ikJQx93y0lqdTE7pGixkvrs7LJYcYonM0mVldXUCwUtfuSlO14037uZfNGqZTsLn0AzpG0B4Bex7QOhY8CxMXms/Kz1CKT1arMDl+r6+t6Xr4nbDMFM3yEiFBC8MOZTj355BcTqhpkslJFGdDB4ETa0vZ6HQ2aaom2iu/lhHJgfJBQY1IX3M30SD2Ei5Aq7DE93xAgqTEP7ai+5Xi5d08JplXs9xP5EXxY7cApk9R+zx2gQR/JMNEC8R5JYiGWpCexHVEsFTHw8IxmI5fNabHtfnwiap8ChoNEO3B9Y10LMj83p5+7rbZMVofOkdtwOUU+rjATw56ZQfkrFNi8LUy300V/0Nd9ad/Hwz9+Nmx4q1GX2s8Vzcni83CMVPGcf96v1WhKC4bDG+8L7ztsdcyjaVWLKjS2Z198IqFNkgT1uihkcpK8YWKhQKgLTjofIn7mLih76KAwhwvsNl5T6HFpSLWkjB6jS608U9nOtNSSpLvXe02IRBulsML/ZuaFXrTZPE6IHoKeJr33rsX0nFhei3aWO4LPxWeKUIy7k2q81W5pJ4a3TO3DBdGOTZuqDDVqiwp0JVR2fwvV0nouhYa01VzU4RCFcmm0q/nMNCvhryhUpUD7HAlTGPakbrm4IQAjjZBOj6KWcDLNL8iNsIoILWOueL/Qlvydnv2p5x4RqFIulc1uwzzbcqkgCTdny8IVOSeuiqhCQqJ4oXBcQm3JexwMMOngQ3jo3FUCWuiM0V9JpxRiUUVxYSOc4PWnJyfNi4Q5TXpQJCjkC/LaeX8+JD1pxrdcKKp4TmIsFEO8drulxZVJoK2mk0YB6nYNtODOd+eQO1iefio9MkXUAAp5ej20uh19nhM5HkoVsjkJlRwlmqGUCW84TvGZiGBoMrtde26Fn7Is5vxyTOHAUaD47KGyuXBzc3OvCWUjnAuVH+qb742/6XpPP/eogkw5LcMBCrk8mrU6si6hqbQF5IWCxb5STZykUsnCKk4Mna9koAGN7ARBAvfeIzzjoLk4dPT4PqpIDmK7XhvFvfzM7MwMWu32KKzLc6L7nDhDybiLqRppTkpFQ6K0A4e07ebwaVe4g8j7Npst/Z0mioJRqVb0lYLNC3KHc2KlGt1eT9BLdmSO9+ecMIwUltDrax6klRJaDQN6KMC8Hk0HJYoCxleYNOogaaFOR5+nNy6zZ2/D/PzsSKOG4JvDa6/xWJ6fD78gMA5uAqGh6YzubethplWLzZ2hsCABOq02qpWKSSehR/q83ClpAwG4GNyx3DGx66QmcqZqAjyhMNTq9dd486PY1uFBugU0B4VSUXZ0HC0at4+h8kIoQ7VucXfT4XEAQ0JZNGiXoZs8dtdMXCyzm4kBNPTUM1TBpgWIehEmrUwY3KmFpOYo5PUzr5dn3I+UaRIHXei48aXQldfu9qShKFjTMzOjiGZkN31M1BS8PwEbLUqhgEa9gYmKhad8hWoObcnn5FgVkfR6Ei5uHL4/5t6wCEMWBU7Rdxmak5h66tnHkoBAOVmUODpOmXQKDC3MVqX1gFT18pZztDe2k/h3gg0UgMCF+X6qND68QhXChfLOzRSYM2UOoL6nL0CwJLHYnrY2Yn/6CozZOdGESTWRdK40Jj68LZjtPBfIlMW2HCvtOHetoNax8E82t0sVaVJvCF0GRPEYslBI+FwMnbhr+ZwUBMW57plzgTkHfF5BpA558rliXqYqVY2NWobCymcNDcdn1Wd890tTMqZniOvQzfT0tASJG5DzEoJuzrAJGsdvttxQtRBwrolpV4tkUi+8/IwjaLsgCgdEEF0OBBfL1Qe9VvNg9QtHwMzrJfTJRaEKlQfoi0nEZ2NzwxElG8y41MbgLTGRlwoM3Jzf2QLaAyREy2lfAallhm2cVH7WJm4gf0A+RD6vhSKerJ3q3jd3KLUBF1DXSlnSRzsjbQ6p7bAKehJYe1ZeK9RqxNpyHtMGJnEX8sXvhTJms2hw0YQZ0GegYAwVj4dQclEnpyYtOeTTyvFwiiLMpRAqWnL7G5uEfku9sTNyOu3vKdn78MCZhyBIQ8xEavyZF59OtIiZFPIZokwNvbndaqBcKGEw6KPoWLW8c0mK2Sg+kOBFd3CUpZmYGDkFFBpqCmZcwqYp5u6YrZH5cODGMjp5CY2841xOmoVj4TWofQK14wSGdqA24WfDWYoIIkIcU30ptDud0b1kagbEx7N6BoEghCzTad2Ln+H9+BniCwZYDLBTq7lQM2IxRDGik1TWsk0Ubl6bfoZ2snvcMZ4AP8zh7KM6NWXJIvoXBT4/zUxfmkJ+1MCwBjqTvP7U9PTImTREzoQtwmD+bmS6uhQUcxilgV4++5KEiCBARmrUEBxmcxT0p2jPbUcRXOC2swU39IuCwt9x0gjtlcplhWHh2PDGdQL8zaYGPlGZ0OcD2aIzxJ/lpPCaA3P0qpOTI7+B15eEc9CDvsKi8GojpjR1Y1omJpYIFe0bNUCn05ZfEF5xqG6ZBU9cUBtQi0i1e+aI9k8qME3YNJGGKJWKSIa2kLy/wKVCVosRjlK/w4wefYMsCDYF3Mz3M2oggra1tY2Oe/Czs7MygxGXB6bPZxF27iqeP0sQ220JFneurunp1LDdYSIVy1PLyWY//1TCC+RyWYM23bGhyrTQimogh/Qw0c7iwwp6c4mykMrsnh6eNtRVeG1nR6B+2DA+CCVND5LQqelJYmWvlRk1eJYf53hGgMWQKnoXiTJNZHlzLmAAGgrhaNv1ecPCeT8JL737HLFuy3QxxuZX/p2LaGAPowWOlwtroVOnZ37G0L3xiCzCpvO5OW+0n51O10wLkbY0Q7WugKq+A1S6n4dk/IZhF6OOgKQjvOQut8RMSiqcY+dzxqbgnEYoK83nDhqvR/vOr1wzCgId5Ugppx596pEk0Cthub2+FpXOkGDPrCUMUkyMM1HiMabCINlXUyN0lCSBvnDcoRQMOkemWgwjpvetzJDwdMavGUkdFzqIArHLLRwkNErEzAAOLgr/zpBJpoC73L3rVqcjIeHc8p7joQntI69BoRHSlBhAxPHH/ahOI1mTTpl2IronGzow7TaO7UcsbOrUEibUVFqklAMy/S7o4kWem8/ATcB5irCJX/lZjpfzwu8j8rFM3FDzzh0aYaG0WJ+hZl/+CZ+DIhs+Q2g5aVHOMX2OrzzxsBabEs3kAzOblvUpyIYw7JG7z90c6kJwqKl0hWeesjTPkHivQYMCMnyyeE3loxXSEK60XTk+6GBtmP9HreK5Y4kZUKvtaLG1kxxk4b1MJXeVaJAQuoaIxRMY4lkrM0kWr3Lx5StwEvs9MK6mA0cVST/DQk8TLu2uMUcp1HVMrrJ2SSJvXlEKIxJh8gyxnGDhmTV+Vo6TmxXZW0LGLoiBuMnhYx6AGEOwcTx219iYMWQmMaITwsaDwUhg+RwCv3zTpB5+/MsiL5hX20POSQv5vDkuXGzFa2RtkHLjoRQnmw+hz7ojQlvHvSc141SkwMM5cE4Y6UWUQEocU5sUsJBCxdF8KAdPtOMUqlhYRc1gnrQtgMXLWak8MyW0nwNPF+6SLwK8oE2kAIQTQ01C28nPa/cS5iyUNEFcAD53eODhcYd9DHAj7DavG3FxhEImtDaO8C3CxDUaNWmY0A5M1hAj4M90TCm4XGgKJ0OucAYDIg0oVQAPYWeaNUfslDhyUItaMfyY1GNPP+pMFYt9mSDnhxrNuhaYzgWlqpwv6uE5iAjutbPH+Gjc7bSLyiyNATDSAo6XCzcfZc2C/ODok1N0LMzi5Nv1OB6OY2enprw3BaxQKJoal49AEoGBJYwciGLxPZxkqr+AGyNRMA7YRMxLdWjYQErXpSaIxYisGxcu8PtwgGKxKbTB6qGm0AJ4WBhUKQoRx8+IhQIsP4SIH59xLEbnNRk2hRMs6Nk1JXludHjDBNIp5Pt4T3EISH4grE2giBh8Pi9TKij3iWceSyg5TGVyMFnu7I57fz2qtJYgSdocTly+UEK5zLQl1bqF/nzI0A6GsBm5kDtcUF/CHWuYeAAInHCCFoa42a6MGNESFvQwzQwo/CAE6ULEh+N/20H8m/JAcro0CQRcGC83GqOxxU4Nr5XPKgH0JBCvx8WlL6A42Yl9kXjg89GX4c+2aJaIiMWmg8YF4hgopAzBNzc3R7loOYtyuIxXJ6zdSYYUNGooJm20OMp7M09uiKRsuzuIyk0QtMmksbOzbSEI4+uJsogYEcJFXB+OM7GD1Jce/aJsNrHtGj88HEjd5tMJup22EvrJYIB8sYRSqYzSxASq1UmUJ6Y8xKKDYyqf6pA340LRVlG1cuI6XebELbnP0IYTJKTO0Z7AfkfeKBGxXneESAkJC9za0TeaAJoMjr3bY5zqSBi/IoASU9nKjrmpUa7aKVAUXu7+yJ5xYiIk5ELyvzYA05m9rjhoy8vLyGWY5m3ImYpEBdOvBw7st3yBzBnnxeJ2vm9udlZ+TrNFUqUJI22tOZ4MpxjimQOby+cUVnEHVzwCoqqTQJaK0mB8z6WLF0zbFkpm5sjedSda8+Kw68hmf/mxLyX8ZaO+g067jmGvIyZIPmcTORx0iOojRQaGXPoicoUiKlML8gRJdqA0kiJEOHUwNFQqGCfaCV1yy7bk/Fy4cAGLiwvYs2ePecEOH9KeinjgryAdctdzh8euNrtkSX9OEAkKVOMUDl6P/zlew9oTQY8kSWSFtqVQKhSxtramu3CMAUhEJDCeOQo1zK9rq1c02advuwOf/Ohf49a73iCHs9M2XDoyf+F/MKdgmT9T54pcHCfgV+IOnLdxti43bbtlISIXmxrXHEFuImozmxyxiJIEa2uGIzBvwfmi3S+VLWFFTaJMpUgWBqumHvzS5xLyoNu1bQx6bXQb22g2ami36yCLI5fLmFpk4l057RQq1UkgW/IwKytUh7TeoiQsh3K5guGgj1azhYcffhhveet9MgecUE4+NYFiWIVK3EGkPNmDmUNkHjOFicTDRsPIhJxsqubAyvk3OljdbkdmCJ6WLOSpRSioxptmOElSgBZ0OJR65cQyAgmTwPtywng92UDPpIWD1WvXsLm5gTe+5W34o9/7EN7zDd+MhESO7Z0RHsAJDQHu9Q13N66bRR1yNDNmvgwhsx1Oc2eQr+EMNJvUKPSsFW45Pp9JG75BU8DfUROb+bHsXIZhpwSKiaqszKbRr90UfvTjf5Vk0n3UNtfQbzfQbTN+LYgmw1evb+nMtHO4h4yrBZ4QB88jTbJDvojiRAXF4gRKpYoGJL5VviDItdHpeVrTmBOBo9PmcMEIhHCSRdFxZC5if+4+Tg7NQLvbcWpSRfE3QyXa2Ga9qc9ZmJdCtcpkRV8U2vg9J4PcdArG1tamcHZOEjNh/EwQB8JciF3rW4mfbTS2UdvewA03344/+59/gG/51n+jzygJJC/egB7aawpKs1l/zZgsvcp8g6U9RcaUo2lzIoFwX4S7lbtaCaLQViOMwVk5bhKEySeGFWTyTEUXTJspbBsI8qVzq4TLX/zZf0u2tlfRqW9idqqCen1Hu6TXG2gnKF/NZEQkDpwJkmT5YMwDTyBfKiNXKCObLSCdLSKTy6BanRKVaXpyGps7dUPcFN7Q4zfHy0APc3I4mIhZd4n+fVQqEyIMcFE2tjZx9uxZLC0tKQ/Mscnm0oZlcyjm8zh27BiOHz+O6ekZdFpG/Y3EA2Nnzjb9kJ3ajpH0U4aARXjEcZjGsR3HCadz1GzsYGdzDdfdeCv++i/+DN/2r79LGiLoxeMevj1P1xiwYv0MtYvDJ1EWjQkPX/TAsoMsEk5faDja+OAO0P5qw4CgEfPvpEQXjXiS92oRYhTOy6P/QPuukPnDf/rBBANOWBubqysoTzhJYWjlJ5Q8euIcSHjc4chIEDI5qZpMtoBMlra7gHxxQna9Wp3GxOQCElJkCcP6i+GdqjGodpBCd2ATzAdReU82JwDlxZdewksvvYS1jTX9vecxcuzWcOzGVfHoHtz5JUYPBczPzOL06dO44/Y7BOoEZYcLFHbbgKTirsOWSrQjDB2DdnV9Yw2HT1yPhz57P97xvm82E0LOuUyMOUfhW9Cho8Mlm8xQivj5iPtmi8fn5e/DmVVenqZnQAEzDrrSlA6bCqyhqePadNoCkoQRgMCNcpNmNpywqSSVo2rSJb/xKz+eFLLMTfeRY/oysbonVmGYnbGgPC5CO0Q3n1IXjpI8cd0ASOdyUunZXBmV6iwW9h7FEAa+iKtFe0ywwGNvARwYKmy5cPkSnnnmGZw5c0YL0uoZm4NaRQ/ioVKABLHYoeqCIBDhEgkVfHCKFBedCRSmGMnEvOmmm6QFIg7ns0Y+X0BFwsXxWjKyaTZWsbp0Ea+756347D9+Cm++712iRtEfMNNjfLjIm9PTjjy9tJrnlhU1EATSHBAM4WLtEhW5Uw1MIQ/Acp00WSJe+m4NoCSfI9RMoqcnnpwzyKRPVI44XGj3+LX//P0JbVKxVECKnGXmdJkA8cUhmCV97xmeqMXiLjCuuZH7hCwxFOoPMTk5jUw6j/LUDKbnDmFyZlG5XQoMUbrI1jIuZCjz4osv4oXnn8dOoy5HLZIe8mYdirUFNI6a0Qu5YUzqRy/BmYwc7DchFBa3GzrHF8fBsIg7l/7I1NQ0bjx1CqdvuUVJlYjh47r83M72GlYvncPb3/3PcP+n78edb7pXBX6tesMWeWglReZMmXOpHcl/TvlSalh+gKlxIYb8zMDoTBEi8omocZjgiKcbkFYfxZBD80+4QfVMJC24phDsyhwFMQg3vYFmpn7xA9+TCIhPBihmWQJEN9/LdrSjzdBzNxIrV/VleIeUfDkkeaRdBXECaZyZCJia24NuUsSpW+6SNy4MmA816GNlZRVffvQrePXVV9Go1XVN2mYLxQzgtwW1laMW4WLzRS1iEmsPPVLd/n6S+cY/GzYw3isChvLmNE/GvEwPWVxYwVS1iltuuQWnTp0aZfc4ofXaOlYvnsPdb/46vPLyqzh2/U2y2TQtlrbkeI3kwBeflTl5YeacI3rVjoFHrK9lF2c9IyxD8XmAJq6OhRYWC2hRZauuwoTF5sTSzj4tUtkULoOxeyq62N3ZKaR+6QPflyhWywJDJh6YRRrS1hhFKQj7uyGRTbAyQp7jNpaG2fRR2pDFe4UK0vkqbr37rQIWRLYf9PHZBx/AU089iWa9MWJNWrxrFZ0Kl9xWxWLbw9kuEanPvW89rDMzYzEJqkilxxZ3Idjd2TZ2qVenKvNnyzkbIsg5IaBx04034fbbb8fO6hWsLl3AqZtvQa5YRaFcVdIj8TqrkTlIGS1bfgSdUa6E72gOWz7JWHgU8KuhjtSNxgW0/IFlBM2AkZJlSBsdM1HFXJOEuFui1lBN2/l0DFmk6MLxyz/3/oQDK5XzSDn91x6YWbCWFps7ke+PhAM/Ssg0dlxUUHCHh0dN9d5Psjh7cQXf9h3fJ/L9o08/g8cefwxXl68YgDJWSx1o2jh8GQscO9cEjjvbfIRQ7UNpZ+On0QSxIsScGtMMAlrGXiEUIUghWJaZM3iSU6a8fS6DifIEKqUK9i/M4NSNN+PW2+8UM1aOnlivu4wUwqaMDOhAEZMWS5Z2WaQI2wzyNZzRqw3j5BAurmWwGN6akFD70L5TG3EjjFBGpmhJn/Y5ZMREDSyOn7Sikys4D4Fs/uSP/9ukpKJwMk4oUgPk6FJ5WQztIyU0EhvipzG0cIaJr7iQLKnYtNVqK8eayeHVy1t45zf+n/jkpz+F8+cuaCe3O1TpVpyuHUYO1oi44EkT7TjPJXsFRnjd8uG1K6nGBhh4sZyx12yhtcjK8VqJsNlHI7jF38eFaFybjAtHwKb58gQI1jA+J4tmfmYex6+5BtccPmDeL3qkfouuJIFNzLHV7vTiwVjgKPYzgQzv2ahFgmY7lsAJuJNzTY89dr9COdaBZ4NGxXsa8ZGOXEC8xrBJI0XYlvyBX//Vn0zajQYmq+Sb9QxtoipKvG56wNJQBu4GBngkotooedJEZ+QtkqFhD6b0Jx2GXBk7/RKefv5ZrG1uIDUw4iCxbNpk2maFcz7rsYBhm2PhQtWG6chI4o0LpyyYCmK4iJT0XY41d7+WX3YuhVTGhGfcnsf3sdvHfYBIJ3Lxc1TtBZL3c0bu4KISfi2X5eFP5LK47fQNmJmwShBqiBFU6hUZdLgshbtrPhgDBz4fwEqMyWrJrALGVLz5TwRvbOGNI9DvGRaiOfDUcrBc+DMxc23WD/3mB5LN7XVMVSYsC6UkeQqH9h/Bvn17MDU1o52aLVWMJeElran00PK+nabiPe5WOhgE8pP+EINCFc+/chYvv/yyUpO0J60mHTDzsBV6yNu23Rn2OB6Uv1eO2RhyI0+aP4loPyq8J2Y8MJanY+KBfAnpc7LguJMW34f61jXdU9+140b0I0TJF/EDZIj/M+WbR67AxFBJDpbsvfyeDMrFKrKpIfbNVnDztddKEzDC6QtYoa9jzQqIVyszSIoVee6OM3Ac0nhjPooVRXhRorho1q4EKdvhUTYdqePYHBIW2vVg5Xz6H/4k6XaZ5aIt6WN1dVWkAuKvlCLaHbryzIpJUl18xIPOpOTFmlonamRgQJLL4eJmGy+9+KKcLg6e3mGzaYjPSK0ZlVrvsV1kYU+kN7ngI+ryWDWE/C7PiZvN4mJzZB5aOcGBJsfE3VKioSliYcMsjNvzEDZG/0aiMEdIi6SEQxHFUkVZQC4UVaS0U8YBGAqiV8jksmkUc1nMVSq45aaTgobTXpJLZyvoybLPo1IdY+2qqsRLltR1watCtEPdQeYGi9DLtoQ5hTJhgp4jXrcwL/UXf/RLSqdQCsx+GrbLeqSwlLcAACAASURBVGVKEFWFpQB366t5MzpYVD9cSEuRplApl5CvLqJXrOCVl7+K7Z1tT/dZxobCwCR/qGsuWDgY8RASHKFK9PAt8xYPZ7nrFLIeUlAABfprt7CyMoMBQ5mITp1HF5LOz47b43FPPDJc4dD1B8zpm2PFCSSOzs8TFqbJylcqUum5gvVqSWjC+kaUVIHgwHqqsFxI8zrsygGeLGXx7ne8HSxl5D1VvizqtFWrBpUrtJIxTswkBMxqxY6SeOcAmh/i0qy/8dmiPs1dFqR+4xd+ILHuOlbiQlBBXQdy5FSToGDeLKmzQqpUOG/0YpHbvc0EXaFBfhKl/dfiqYc/j3q7hW6LjpgJCz9HDjZBei6MFtE5zrHrAgkL7jYHH4BNCIF2WYQXopsx+LTnlKOUIZ7kxQgeesX1YyG/NpwLTRM73cIWCwNDy1CdcxMYPFxEkiNzp4wkYzufQsD38FqCdj3lmvI0roiVFM52C1tXL+H2G6/DO9/5Ts/W2diJZ/Mlb97JFRKUsZKrCKtIkmDVjsHYHoV4XxjLqRv3PIAcRQS/9cs/rG1n5D9ic27nvPoiiuRMzbgO99KfiANbrR0MhxnsP/12/N3f/SUyDnZQOxiNyJiTzDoZB4w/m80Sb83VdYRtob7DBsm++w4Zt62pUH9qCUVfg8O3/HHs4PAFIqQLJ2/cRxjH2GMMDKG0WxyNE1qo3LLVUTHTx8RPJl9Chg4se9Kwhj2VQb1hiR9OGGu4FF4hjXTSQ7NeR7u2iU5tE//ym78JJ48ftbptItxO+DAGi5mRICMGrs4oRxx4gkwwGFUl6iRDiMpkcxuVNJFdUzLlv37wP2ixVZfsZD05JE67FewmgMOACM5vgP02EH4uwczR2/DYc1/F6tIr9neVsUTLJ7NrDCcaDcKmJDdSEMx+M24OdR12VWqIVZNy4v7/VYzane5lWu2MIUtc7FDX4Wz972x0/C7s9bizpmuz84SXB+k6LlhRCWI8vDzSuRISpRfJiSvK8TThNAezXGE+voE+bWmvo2Cwtn4VrfqWHLef+g8/aowez9eP8geROxBl2KBYsW2UhevLUMlNUbxOyNXyF7wW7z1OqwoMI/WhX/mhJBZUgIX3BIv6qmBXWALe0pPuH5tXyf+dFvLH34L7P/a3SIYNDZxMC8F3TMnxMwJDDPK02m4Lk0wN79rmcFSsPHfXWePYYkxRQWnjME63TJbHcKGmww+I3bp7bbNv8dz83jJ4RpDQriSvzZEv+QxU105CMNvpoU62YOYuV0A6V0QhVxSIwQVniljz0++jTnIGG24NE2ytLmN7ZxXpwRA/+1M/6R0d6MgydUmVbpskiBARchl2bhiZxeduucliCQfWKckjs0aNOCTjN4/Ub/3iv08YQrCaIfhhu2GPYa8RAoUDZ5JvO55aodnroDZ5E557+CHUayvyUoOcR+FhJ0LtdudHEVMW0N8xcgFDMKk6955t4i15Eeo7FkEL57zvWLyAH9NZW0Q5bWMtu8a97XD2wqEZQZtj8Kny7EwFEqgcYdVWshTqn0V0NqHuw5C/njMiZrqQQy5rxREZr4ztscojGQgf315dRr2xjnwqg//4Yz/ila1dLSQXJgoNZJfFErW+K9FKLNp1EBs3pMyRNufnGZpsXj2/mgYGUh/8T9+nKk5WPoSBskm3zJDZM8szx1dzZAylYrhEqtLmxLV49itfRLOxpsExqWDCYzsyYL4g9wVRn5+ntgjnKHZbnoUEASOSOapWGUZb4kv23MEVLTpBBu4cx8/HwZH4Pr4K2Bgj/MeCh6NmKt18F4Ieso8Ou45/TuPwWD6XLig0Yx6/n5D4UGLnS5RLJEZah0JmyQrZNDZXCRevo5jJ4Sd++AcdLbPuipayNAdTIIwDMOGoKUHkfsS4mQptFlrMwBbWirtW5dxxsWUPnPX5tZ5qEP/dr3fyn4Hz2o3suNDpY/KGd+Lxzz+AixdeRNY9VO5wMk0M6SJD1CoUgjhnHja9cgM1DB40ocupoJBCZa42Q6qAT0cPOQb6K+4nNjDWqoPPFQscKjoctPHnDOctBM5UqAmVFbfbDhnVTHmZrqIRvx93eIoOWybHDJChXKRZFyc1hiafvdVGIZfG9toyavUNlHJ5/NSP/ahrNIIO1Epm7zkHyi94nbnh6bYfd5MlZsi4uagNhNx5HkB22pHMqC9P/ebPvz/hgKluwhGKna3p9fAodpOBdmzlZIxKJgJanT5Ofv2343P/9ABeefZRZNJUw6wVtvJdAhGhsg0T52TKuzDKMLsVhN11hEwqyEOvcDYi2c8HkkMXjXr4wKL5WLw5WgDPzH2tGh/f9eO7elfr2K6WgIAolJVARdGinM+BJzBYo6XSHysglLOWNgHJ5stC3bhjudDKQPXbqG2to1nbUi79R37g+1+jrYLepDVx51g5ctcsMUYrLdrtLxsmRqGqGEAUxF1QSprhN37ue9VAx+LBcFJMYsxT3m2foR3mHYXDzhK9ajVauO6d34Gnn3gWzz/xJXQ77NhgHuHkpBXDGxZuVRoR+1kmJ6V8dixQ5K3lhHmMKiKe57HNSfOiAW8UQGecjk/kt83W72a75FX/bwraQ+XLprmDE9/H5JFLxvdxh4emkJD3jDOnZxqShWPv0SKl89o8SOeQVTtN443xvflsVqyXTquOublZfO93faelI51PF4Idv4tx8e/jYwuTE8JhPpDVltNB5L2ClxDzl/qVD/w7lexavbEjVGNNVqN6kQ8RN+CFFhYWwBYQxWIeSSaHzuQJnLu8ise/8KAexpy6IeYXZ71wwOyWhVKmqqimVNM84lPvdn+IQgOOje0raYMCD4/sFheedj0ctkhphoqORY5F3Q0jvZPDGGWY4+JzRQgY6jBaXkdnhQA4ct5zRmgZm+8RIVSM7w1o046sSWPSnzVGSqrLxj/b4udff/11+OEf/EFfbGO2hJNq/lHAqJ5p9HZlaTmHDDONYxa1cdS6mltH56h9ogpUc/BLP/OdymczbolYkzsnVGXknMnbYq8RPvSo1ssTCCwZquX24NIO8MTnP4Mrly+OgILyBInwjEENFQpEzXZL3hrTpq2nWBD+xu1sOGJmUkIhW2Jf2ACT/DExY4iZdp+XvgYuEJM5vtPDHkc0EL5DaAIrKjRGy8jR89BHvVy8dZeySwlZKabOuU4K1cQxy6g0R/dXjqAuuPRd73o3/vk3vHdMjTMnb+2/FPJGaOpOqXnf5mkr7aww2Xh9Rllwe27fjHiC8WypX/zpf5swSJeKYTG351S5uATuc85bjpCF8bEe2u1jmlNNzzFVwvnuNB556LO48NWXkMomyInUDiwszo2AFAvx0t5vu6ydHdpDu9ix8NiNoY7DpBAXd1/JAIxUImGx1N5uY55Q5fE1JinEJa7Pn2PXCuN3vH40qeS5ec45FtxqoS29Glg2+WEquqcL7tGCqWAjTrCXaTTwEVU6ncKHPvQhlUiHmRPbhw7pWBp2V0CtBp73NQ3rFC0nMHCiJdzeL2a0+B45aSwf+In/OyFXiv27SbpXB6IRMS9tOLSyLN7wLpIQUYutBu9ZdIcJznXm8ORXHsa5l55Ft99GOrHWUlNTE1LZFDcurrzMPqE9a0jL3msGtJiHHwAHB8hdoqY3rE5UV0Dz3G3X7qpxg3stsRI7OhY6zAavN55wGXfUYnF31WhMqoFIRtm1/IBSvS41I+dJZLY0uh0nGoYdbvdUkkP1ru5L0XigVMQHP/hBoYCGVnr1ihMTuKjGOHGKkYeD+tmTM0ZiMAatSIteVGkIk7FUhcwpu5hC6o9/9/9J1HzVS2eEgdDekBJM58JPGMhmmOVJI3EUiQsshIv9vAg2II2vrnbxwvPP4qlHviSCvvBqVmeW2LzVPPKYVLOPhhoV8+wRYrxyld96OBOLEwLAWnH+jTtZsbtHBru7w9E9j+3Gw6zxRRy/7tdqgLh3CA0xcj4rd4xahgRI4YsgJ4222Om84deElookje1QFjQaF+/EyWvwH37sx91OBxXZulOpfwrDWmbt1FLL1HIIp1KqhRyGHWeiOOql4zjU9M+aBFohgiGRCls/9td/mBTLRWTUSwQCBZKEKTfr2zGi73oFQ3qw60QpNEmxwRtj3DSu1od48atn8ehDD2B1ZWmUiy6W8ihPGJPFvHEvuAtb64sbPkOYknEHSw/oD0xvM4SGYyTGzOvGZHxtDB3OllKKXgfN7yMBIgFyGz+uBew6VuhOSFRC5zy34I0x2aNIIW190MI+mgOaRTIIO2u5ezstIY1f//VfwczU9AhsspbfFs4JKQvbzHvGbg/AhbaakYznrpW/GrP1u2RM3ziujVMPff5+IX9q0KL2y757vGwm3H2Lei0nPY4hy6HxdFo/yeHxVy7jSw/8Iy6++qKpmEwa+VxWhQfRp4XccF5OdUjFDLpt6xca6pkTHs1aaU85iVTz47tw3KabJTPHJUKRWPiv1RKx2/lc4/cct7OKSZ0gEOxPYeXBb1NDH2eQuhYZjzLsnhmFWeY505QbCklG7Xd/93fjDW94nXPw9FcRMGge4h7RrYmXFzVpnA3rfPQe07DUKS64chIpcKo5G8rsGcnRk1kPP/JgQk/R0pykYxqYMALhnWLbb1uXWz6keeNx8k5KD8JS3VyuhOcuruIrX3wQLz39+AgUoNQyfjS8mXnznpAhkeDTAyR9CxnGqzPi4aJOy0AZE7RQw5EsYYO+r0XG4vOhHcIPCDX7tSp+3L6H4IzfS8wVz+Pzmv2ehakhMCEs0cFR3HkdTZHHgYMH8KZ77sGdd95h+RWRRUwTRe6BZkkOn0cQ0UslFt9Ewtil9PLDWbOMJVG0XWbqeMtt81E8qfT5z9+fsBMv7aHVPRmfigNSAl0XIqmcRXQseLOeXqxgZH5a2DbhTZ2pUcCVtW18+nOfw/NPPKLUpXUpsm75LMfhBLJVRKdjvcJZE8XidoUT8jDNQYtJCE95F3TZ7T8mQqEcOscH8plRV4TAv3fBEXOc+IpESahsmYgxtC3MQGiPuHcsfpiC2P1a9HYfe/fuxfu///2iHhsM5Pdy+rAEMG3PZxTh3TGxr7uIEuwU6Y3reV+WRRlgYk2AeS91qnAiYtC2rJWJbRoCQcIlIivorcVSD372kwmzVjqRJ2vdh1l7FQDEoGt4axSuST2pgsT7blLd+SEtjDFT6QKefOUM7v/E36Fe2xoxIwnAWO/SrOq2u11SZ62WizaXLzEyHXCJiYoJjh0+PtFy1EZJGh65YDZzHIXiIkZIFRBo7HK+N8xULGjYXA1ojIgYAjCeJ45dd8cdd+DffNu3e67AKjZpQ6PG21SpF+2JXGmYugmZVW8QhwgnkjtcvD0nDHLhtHO9k4L5GAyTdxeVi22JKzp0Rhahn0EBoGoX+vfpf/ibJM3QqdPWLstn85icncYLzz6FYcIwjJBnFXv37ZHtaNU3MUgySGVYrZlHZgDkK2wIYwxPqphXlrfw9x/9G6wuLwlDZ5E4ww+q6Xqt7g3r2BfNeoMOKInOlFEI70kRIy8ECXG3VktxtZzH6LliNnZ0ksAYOTGw5JjIWAC+N6jIdoSUYf29riF8/G9CbdpGCQ5f/NAEHCfr2n7mJ39KY2ZhgHqjD/qqTbfEhqVbWYynpvYD48rzFa1GuLBEIlUbzoZ9Y3kBnVDk7SrDbBCNMzqxaYg0mUHhs+ikBeMPcvz0j4zFk0Lqr/78D5Lq9Ax63bYkgdX611x7Eg/d/wkcP3EKi/sO4+WXX0Q+m8aBw0fx8tOP4/ipm3DxygomJyZw6dXnkJ+YQc/JJCwiT+XzuLzVwSMPfUYdE4kzVCtV84QdoCB0yvBASJDiCqtdGn+Zat/9XahNBXoKKSJDZHlmkiNjUUMtj9vmXe+eMazVnekeHpoY08N7sPjC8prjsWqo0sgw/b8/87OYqU6pw7HUvldi8Hk4FoavfFajEVGT2PtCg9gzMS9hVCRRmdzzj0NtKDChUaTxmPpVBMDuzz2rvuUpB+xVquY6lofv+r34GYFVH/nw/0hm5mbVe2t6egoXzp3DnXe/Dl/8p0+qo++RU7dgmcXvVy/h+tN34IXnnsDJ625Coz3EwsIcHn3gozhx+s0oqEVFHfv278fTX7of5cM34S8+/GEsXVpCPp9RO6geC/ac6cLJ4aFkQnpiQcc93rGFJl4VvTsNVCHQE0wWS4wYkGKCQVNjDppXcnqXYOamJQyBKbN6xc/90G7lzus6Bz1Sq9EiOrEMHR1F64OSYHJqGj/3sz+npEh446ERgnI1KgOWX8IerB3tYIJNpkms0Q0PYlPNupMuIoyjsLIxACneuXzBKkM8VCQMbfQuo25Rm/R40kGpKN+l06xbXThbpdCGs/PC3MI8dra3MT+/gLOvfhU3n74Vzz/5KNqNbVx7+xsx7PZx5sUnceTkDUpyFEtVzC4eQnlyAk9+7mOYmN2L/Ueu02IfO3YUjz7wcUzuO4LOsICP/t1HUaMq8dZV9DKFJMkeGUU2asis04QdTmbVIl5HNebIjHunEarJ3ku1pcSQMTVoFY2aPDXX3c1ta4d7VYWS+4RMM1YjxYlnSMjvdz16i5F5P3rXFk7mVaX5rne+Gwf37hsldsLBJFeNY1LbixZPTjCba9i4naQQfk803+NX7sDwJaiGubhsTBC+C7/yOjqZIA1t0si9B6N0e3vHyCNk/uq4Spbx9pD664/8fjIzO6u2FWxNwSTG8ZPX4crFC1i7/CoOXH8bFucW8NzjX0B5eg6TlUnUG01cc/I00rkMnvvypzTA46ffpAXau/8AXnziATRrNRw59UbMLsxic2MLTz76EL789BksXb6sXWGevrMynMkSB4lG191oWZl4q0h+jhQqPgiPfeAujxYUVu/sPcZGoIsd8Cq1SJUfdc1OiJQqde+fAIXh60Md+CoMWiR9o/bypTiYcbP4vEAubQ1riO2Hz3H06FHccMONygqye1TUG/EZFNuzOW+vp13ISwVMSgRRi+LnpfCrteMsqgcMhZj1d1w0CZu34OTOpkIzSDnB7MysasXYnSoO4su62Uj99V/+j4TF6LWdOqqTVaxeXcbhoyewvbmGK2efw+yBa3H0+LV48ckvoj8E9u87iq3aNvYdOI7iRBlfffJzaOxs4/ANd6HEHT87iwuvPouNy69i7vAp7D98rR7wxScfwKByAB/72Mdw+fKyqb2BdTgO+0Xpj7CEoQapwnzIyLZx8Ny1Ukm0/Q5YyJN2gbFsmLXVjOI4LZYxHV6T16ZajyTQbjLFD5rLG7NVbBSP7y0c9DCR2kQcNW8G7zn3cNCII3CcLHZg/7SJsp1lwrCM5nHYbSmKoa9jdKs0+sMu7Y4EgYe55Qs2N9T/1g/V6r7Y+ULOGokjjZqKKNVpiTVfbPbXrKPJDlM6Xbfgba0HSP35n/5uwqpEa59cBM+Xmp1flId86ZXnUJpawPEbbsH5l55Rw/mFPYfEpZqc2YuFxUWce/ExbK1cxsTiMezZd1iLvXzxPNYvP4t0YQLX3vI2dSB89bkvoNnq4vMvLeP5xx8fqR9BmNHPVOwV271c5JKfFMDfaZFzu0kaIWV+Qq86D3i2R4APTxQKh8lLYwngMOHCtKrRjiyhEWaBqcoAddQtSr3COXF2hgfbVZl9NB+DZT8sMOQiqZuTzibxhgEOdFBQeF/ZVPfCC/kSDh44iONH9mNl+SoOHTupnnArK1dRmShhdfmiHK3DR67BytUVnXaYKxZVhdlt1sVJLzAbmStg2GubZnNIt1CqamytTgvVShkNP6lPWolz9Vd/9jtJvkxyoDVutzjVmrGtXDwnZujJG2/F8tIFbK0sY2ZxrwSjOr2gU/GuXjqLnaUzQLGKhYPXYnZ2Adubq1h69REMBykcOf1mdUQ899LjaO9sYjs7j4985K9Q11FN5pUyZOFXWtp9+/Yr3hYzxI8nZlTGn6lo1ZMz2l97VaaFFlSnFk7xWlJvcaY2QaOx46oihqeaFN3XF5+2UPdxhzHUvFKq7jCypo0aYZzUEeDLOFizGzNb7xQV5jmGoNjeyZgEnt56772YmpyS8DY2LmNicg7XnLwJly+fxc76KvYcPIyt1VVkEx4ydxUz+49jbn4R68vn0ajtoFouQIfjFLhBymh3Gug0a+i1TdAIdnE+Un/xJ/8lId+Z+LUC+X5f9pDhQH19BcNUGvsOn1B/tPUrl5EpltUMNpUpYe/ePdhYX8ba2efFtZo7eB0W9hzAsN/Buee/qCMo9p28HYcOn8CVSy9j+/IZJOVF/PnH78eFM+fQ7Rnezfvu3bcfh09ci/m5eeRy1sEvuv30O9bnrMQDYZx2LBXrP3Px5HQZqXrk8Qu8oPCy+I5xrjea5zPy89FFOECX8URKNKoNgYmkCSnBStHGkY9RPDiWw+Z4IlY3xGs3JByhdrLhPF/T4F8ybCmQxw7OYX7vIdz9unuwvrKEKxfPYe+hw6htbKDb3NKc7T16E0rVKVw5/zLQazGzquKLfGUGM/OL2NlclZlg10rejzSpEos1//T3fzkR31nF3XYqnzrRF/LoNJuC6fbsPyJbsaZMFoeWRbZYxsL8HkFzK+eeV0gxufcYFvcfE3l96dXHsbO5ganFAzh6/BbU6ptYeuUZtb185lIT93/606jvbKDR6eOHfuKnUW8P0B9aX/B+t62meYwfCXiwebwWiIiR0CnGqhazdhjX09apM7E1j+VxVRFeqcpFaUMrciAwRE1g6VaDaMPTDR5XcMnioNnIkAmNU7WqMWIDsKHNpcPJ8NLOFfXTdrx8KFp18/ddnnnqfcfl7XtmXGeSqZdMTxSmQwcP4Z7X3Yna5oaAm15vRwvOse+95laZ3NrmEmqbV9H1as7yzF6kszwQponWzgpSgz62eYpvZRKTc3uQ+uPf+/kknS2gQM/RWQ18eC5Kp832WAkmpxcUpNNpo//KTZUrTmDf3gMCA66cfQHDfhPpyjwOHL4OxXwJaxdfwtrVcyhOT+PaU2/ULl8+/6zUYbtyBL/727+NlbU1fNcP/LjKaLa260ilzYwQwKF3WSa/LUlEqqCw8RpimGZJY2L/MaYQ+xh2efRCH722N9cbU8uWGrXr2kIbYNwmsqdG+EaJChiWX62Az1pYRIYvgI02QxgnSQaiJWqSw7KMcdXbTYV90aXJEiZ23rbF/vZ9HMhqHRSkPVRTwTH1UC0V8N6vvw95HajXQnNnW4zUvcdulTlbXzmP+tZVdFtNadvS9B6Z1+3NDaBXw9ryZWvik6RQnV1E6g9/62cSNpnLuo1MeUaF8KBaMOoQlylkeUh3r42GmCZZtdCYmJyRyqfdbuysI5cvYe/hU4JXV69exOblV8XeYAjGU9uvnHse9Z1VzB64Dn/2N5/EiVM3Y3pxn45n1IEvLEFVKGPg/wghEzrURSGbt3M1szxkhXGmgShpgjE89LxnXYLZs7TXZN6YkGRXNdGKad37p9dPDRKN9tSvLE+wYjCCcFlxysW26CCl7gahBfg7zoslM6xsmDvbnD5r6MfFEA7gvcKjC4Oa0PF0AF7DY2p+r2ILfc5r5HrWFLA6kcc3vOPt6LcaGPa7SJcncOyaWzBIp7B+5Ry2rlxgcY5M4fzB61EqTmCYdFDbWMba1SWFqRSwyvQCUn/wwf+YkKhAiaItYvsIhhNsXqf2Dil6x1UZeXYopoqU9BdLKFen5KVurS+hV6/JBMzuP475hUX1DVu/8JIWYM+J27G4cABXzjyPVnML5YlpPLvcRXlmDp2etd8S89QXkhk224l+aqA7TMzMyXazl6p77oasWSUoEyqceDaHS3kbCi4YPVnZzYT/DeumqdFB65HedWKAWlzJy/YjLbwgYChTMlCOOrSAOYK77BtpAbD7RFvevPkJ1pGY17TkhrUXCdqQBMd9iPBfDDJmVScPaAW+5Rvfi/SgZ+ZtagYHDl6PHoZYv3IejbUr6LGWPJNBdeGYmgT3ei1sXL2IAR01xuoTFZSn5pD6g1/70YROGNtIkFrERVZK06sp1JvDKx0M+7W0W5LKYnJ6CplcEd1WDTsbqzqFoDp/AAcOHlEP1NXzz7PfFqb2X4vZvfuxvXYVm8vn1PZyYt9NuLTdwOb6ttAuJUl27LhFmgp77Ta5s7DL6sO5s4lghSMU5bWMyyWILhQcL71QCpESFd6ey0piTCtQGFhTpSMn/WgK4eXMoHmKUhAoETcJgZU80RsPx5Dawzh1LHw0UkR49LxnOHcBgYawBFrGnyk00gxjPVzlHWWzeM+9b0C1lLPqmvwk9h44KlOyevkVNLau2rNkM6jOHQZDO4ZrO5uX0anXrCd8Lo+JyWmk/tsvfH/CKgZCRTlWIFKUrNLLzqygM5GyKkURERkzisGWQ5GdFgoTGPSaaNW20Go0QCeBi02MdvX8CwoBJhaO4NCx42g2a1i9+AobV6By4HpcqvWwvr5lZaaqELWJ4iIrJednafG+ERLxIQmSiEbknCum9Pi5qNfm7jOWqhMTiaDpyGg7tkH88yGUk9fnlIywMLA7sG4S2ZQVshMjUNJDXYzICvW0qHvhhoFbXpq7qOskD2kYp2AFeV+dFb6mTCcSKiGMwaAJX4Ff3/2W12P/4qzWZXrxKKbmFiVcq5dfRae2au23CnlMzh9BuWTtvzdWz4JUETmZ6Swq0zNIfeg/fXcigqHjyAmbzbK7AltLyzYzCc4qA3c2VFCQIJPn+ZhF2XpOXmN7045xqlaxsO+ornHlwsvoNtaQKc7iwPEbJCjrV86i3+mjtHgMm/2iuFRXr1wxRMhPD7BeXl0hZOEpR1ZMRx555YUQLSpELz5Uk9eoBGU9eJ4q11RmxOKWnuTCkCnCyfDzNpyDprM0WJbkvdA73ThegpSfFnLUbqQww05D4PUUQXS6fta3lSSHLQ8nLnZ34O2RJo0jKFyVuYDasVFxxOV77nsD9sxO6muDMwAAIABJREFUSkUX5w5g3+IBLeLm1bOobSxZGXRviPk9R1GZmsH21ibQ21I0pANwGx39PvVbP/sd1AFyoDgwNokXu8MdDJaeplM5JDnLVVN9m9NCmnAJ7A+mZCNVx9YWUrk8Fg8eEzy4fPEVNLeuIElP4NgN7kEunUW31UV25iBa2WnVSa0sL2uRGA9zt6lGKTPEsD806JBN5ssT4IlEskHecC8otOwWQc+a0Kd2ijxj8uDN+7bOidYWK5L+dK7YYpMTpaSHs2aiSWyUNxGv5vENwx6dKPY86arUNpoXtPtdMw/eKIj4dajigIEjPx8xdhAX6DyFoxhCbQ1sR2WaEuy3vek2LXapNIGpfddgbnpBuYzNlbMYtLcUmRQmJjE1sx/FiSo67SZWll5B3rVVNlfEgIWHH/rAdyZiOaQtO5RmGwmiUZ6xIQKsGmVWJqZTVmzOXaiOPEWUJspuuwaob22LZTo9u4Dq3CK21y6jvrksFHnx0CmUKhWsXTmPZn0HufIc2qX9SkRs7WwpyU71yyOQAokKtRyn+ubyhosTdaKNJVOTqUL5QGOlM2Ez6UOojIZwqx+uqkn1BjTMGFEzWJ8XClZeuLLial88xqqETOkEqTmfU5iUVnXnyrxpO4SdziCzXJEAEVbujFad3R1HZYjM4Od8e8M6TmQc16gx+CE0//xdb0KF53snKew7dBIL83sl1Mvnn0ONNps59HQWE7P7VRde21lDNunIBxLUW5kStzD1X372OxOzOVb0zZBLaFTBHDX2CleaMLFQQkcTqNk5Y/Gy7IF1sx+q9zYHWChXMLfvIHrNbaxcflU2ZfHIDZiZWcT2+pL6irAJfXfqGvkKXGweDcFqTsbtUaHoLbSlVjmZhFE5JmLcUc9katGQNf7nwgX9iMQJ29nBJPXKEYV5u6fvMU896HfkeCrP7nGwbDeb1PJ0wFJeKBfrzsLDVt83liA7kKJkhjtYTGTQOYquhMYPYzLeqFfRwcJy7pGPtwaC8iGcEcr+qd/yjW9DliatWMb8PvO4eZrP1sqrqG+tWPuNdA5z+46qgrTZ2EK7tqbjP3QC4YB14hWkfutnvt11hpXQBhtEh6MzvFExALnZWaTzVn8sJiSTD7Tn5K3xZKC8nYqrcy1KE5if36sdtXb5FbFVJvccxszcgjr4s3mMSIvlEwpVOmxDUa/LuYlcbuDVlvWx8ETd/dkf1Q84CcZKwkXgJDsi1uq27TQgr57kLlVhuoTaGTHe2sPOv+buMz67cs6eCrW4Oiv8nCRJOX19rzrReR5RgUJBs8pSMkeiEQl3KtOl7CYch89F01i69jI3znc3X4MttqzDAgWHWmeyMoH3vO1OTFan0RoMcejoKVQmJrFT28L60lfR7zYFnKTSZWlT9UEb9pB0G1hauiRNUixPYDhII/WbP/2vTY37ohqldRdW1NmWKo/M0OCpFFUYsnho1geMks42URaCMITIozI5h8rkJJbOP492s4nKwkHMzC5qR+6sLVviYvpa9NgxMWV8rJ4X64fHysmXSiY1iBAn04I6e9MSGNwd3Fl0jnhdlsFGaSwFNc77oAqLuF2qUud/GeOFcTX/RuFmbRuJAqq58lBqBIl6fM2TiMPmmrnY7aYcp/Ba41w3LXQO++yVZJTrqLSMggdreGMLLSrx6IjqtDTD1FQV/8c736S5nZxbxNTsfoVXPDu7sXEJnXZNglyd2oPK7KLYNIxqCKrwpGSmr3fqdZRLk9zZ36Fi/MjcREDPiVD44+CCtX5iC1s/c1pnhDA+ZjuJtJrCMUHP9BxDNoIwk/ML2GKXgc01ZAtF7D10UiqPP7MNZmX/ddjqG57MhHuj6Uc9DW0RR6GKdiorTzpIuEu7hpUTEVP7KLbS9J7oXLxI6PBZomCdpkjtuHg3jdvqrWk+goIbTQLkoHq7jvGwyey9dX7UGVrcJN4dOUgQ/MoIYLz/anjaUZAoCpXrU+5sgwGN2B9IG1uAc17vufs0juxbtM2RLePwsetFaNje2cTm1XPotWqoN9uYXdiPdHZCm6DXb2NjdUmhqDUw4Jrlkfq1n/y/VJ8ttTFWlmq4MGucrMsfU53y1kX5zWHo3QJ1oEqprF1ON39re0tYNosGipOzysisLZ1DtlDC/P6junnS62Fnex2Ti4exmSygM+Ahbzy1hhMPdFpNLabSrCsrQsbUUbHfwvbahtSikKiehU089ti47XZS4Hi1pdGS/MSByIJleaotbbkVHhi4stulwPhscYCLV0+6lpFH7WQ/2d047H3sFEE7etF4YSE0VmCw26dVrFvaZTpq6pC4W8BHLcCzWk7fcho3nziMTqsmBK5QncUij+FImGhpY3PlPHrNGjvJoDqziInKnO7RaO6g19rRQQHUVKRIsX9b6hd+9F8RNbbzPoTC++GnnguWeo/KSTVbpUfMHizehsIPbGOF8GR1Uk1pq1PTlldOpTAzN4+rF8+jN+xg76HrpHImiadfWcLk7CLWM3tF9WFMScePue0aKTU6M2tTCRFmgsjk5RENje0dqXvBlElw2g1vHq9uDApSLLx2ZZza5+UycVipOh6JyMIODFGf6ScI+yLuxskegqrbgrFbuctD3ZN9kuJCC//uW6/vsb7qTGqIaDFioBikGqzVfDaDt977Nhw5ehS5BNjavKjsI9X9/IETmJyeQ2o4lBrfuHpOY6YWzZd4tGNFgkuKdrOxiWG3Y4fJcjMih9Sbbj2U3H76JuxZnEW5wGMgbGcYsmTHOUnL+JlVVNuSfB4xIftt8CV42MpE2equqxXtNDam3X/oEFaXltDpt7D/AFG0JiqTU9hcX0OhmMdw6jp0kBOjIzhZdNSIVtG2Moxpt5totWroNNtqkcm/G1drt8JDp+xSCBMoHAv4MXaptFLWIFYdqRB9x7UQdppwf2AkiqhBD7ttTiNtOyfDW2RFoTyv56Wz0jKEPcWMTsk5ox7ghomW21UeLyV2ib2OHz2Kd73rnTrakX7H8089La0wOTcrz7+2eRk7W5tqaLD/6CkU6FUnJG3WsL58Fjwsjru2VJkBUkZy5GIPBy0Mve1GVwfDVZC65YYDyc52DZ1uH3vnp7BvYdKci2Qg7teeuTmxKKpVghpMORpRwFgtwqasFbPjuJwoeucKHZIheEYlJW91dQULe/ag3e6iPDktQiL9vurCYaxiHgl3sLJUHaUtZZO7jFlbaDUbqO1s6G+M5UmOCOyZE0Shi1NpFaOn2bynjEabJTNZxc/WoZ+JClOlPG6AgsoiCNavjRIgsJpoU+27rUWCjCDVOxiiFGd48z00H96TLCNUz2JrhWR+AnAqm0elmMVEtYiDC3tx/fU36Pip8ClUxpMCnnj0EQlloVpFv9XC1tplgGeDF4ooLxwWKbRR20aztYN2bUtzRH8qW6yiVK7aCcHtJrrtJhKCQATApE2ySH3vv7o3YTqvR8eDXYa9+ZyqCr0/mb7qRAErLdGBLf2hFnl6ahJ79u7RQSqGaLGSgtUQrGe2Qv04TqJa5Yl5fRQqVSFOxL6LE5PoVo+h1UuBNWeKibsdLQ4dL8boGxtrGrg87xbP/zLcOcJEqWOPkYm4EeUSEZD1awXrrM+QjQfAqgyHKFjBCIUsT2ZhgEgDNGEeOAU3OxbZ4E1r0MvPTfL0PyJnLhhWnsPr28HqFMZKtYo98wuyvRN54hCb6LR64gIUJmZxww03jLo+EKmjKfvyF76AieokSpOTWuy15fNqbstoZ/bQtfrabtaxvrGiEJbRMdkz1akF7XpD69qq8GFYxnFIjdP3+vkf+iZtEjZmV6rNCXW0wZwk4b7qprRbtald5z1MlaPyqg4V+fnpPTOzM7j2uuvEqCAIYIOwDj4E7SNVqQashTkkU0f1WcbqFBR+JQOD8XOzuY1+u6OfyaYUB9pP9RXgIgDD2leJBOAn7vCe6YxVTPa7BF94CkBJlaOBgKnvJ59HqVbadfNfmC3Ty7NbnFUlJzy2Vh8G92tYp8Wdye4Kx48dU/NZ1p2RYXLoyDVoNxs498LjSPptEGsvTC6iNDGtkwXjUHoWPfL5udiV6pTCrPWVZdRWz9uclWew9+Bx45HvbIrlQ4iaY2r3eiiXp1Am7yCblT3vd5mOrqtdds6Zralf+YlvVehFhUz4Ubli5oVVAdGjhTJnw20UmV4CKFxN8fd2Gp1liSIG5c6k/TLbbwT9bsfO/5pfXJQ22L9/vzx3kh6Ge06LVkumZiQSqKLIrWq0ttDheZs847vZsF2tQ8GNzMAXcXsKJl+BSRND77Pdh0jypFsVBcwwNOFY5ZiNjk00Z288V82Ja+zU7JgI1rn5ATlk41II+PXUtdfhmmuuwebWGmZn5zAxUcX66jIaNfLF+rjx1rtECrx85ln0W3XNyfz+48gVyzh06JA0DL3xKGp89OGH1fF4Ye9BXL54Dq3NS1aDXZzGgaMnNY9rq8syZdnUAM1GU2dwZrLkBvoZpMOekk6N+rZiciat5KP815//ziSqIuwQUivoppo2NTeCeXczSqPOu+pY7b834ELagQkJP/vLSkkNmaOU8e+0pXSoKCjqMcJMenU/7nnft6Pf2UGjZWgWsd3hsCe8emdjw8kTLQmWtWvmrjWP02yxOZb8T4I+zzmhGTFP2QiJKrLzDglBPxpRguh3iOPmJ+QxqZKy9GppghqqjLfde69ds83zQbMoVytaTFasVqozow5Q3HV0Lq+/5Q70Wh1x6evbV6U5D5+4VZNPPjmdVDsdyMptv/DQQ5jU4Xd7sbWxgtrVc6i1apicP6bUMcda49mpTXaeaongQLw+V54VtVspzWSI7Y2r5tekmYqeMELGf/9F9kET3OMkPe/d4VxsoWVaLMNwhdCovYNpOU2hkhCEuaPO2tpRmJPDybfLqwGxeox6aa4awQzVpyWXTuPU130LtjpsoleX3SNEyd5xW5tb2FhdQTLoOH5uxEIuaqdDLNwiAnnebPQeDVr7xLG9/4rCoYHIlJEGDWhW2pr0q4nyqE6d5ufmm2/GwX3k0PdF0ZXjxRMH+fBeU85Qi1jC6soVHSBPUn5UuzS3N3HkhtO4dPY8Bt06NtcuCTy68dZ7sF3bxpEjR3RSImFTWhCO60uf/zymZuYwNbuIrY1VbC29it6wh5m9J7Bn7wHVfK1dPS+NOzs3g1aTMHMH+cqsauTps2ysr6K5sy56mBrv8Yhp+kh/8ts/4H3QbCFUye8Hh9mC+lGAYyfDKhRLeeMcnbgzVP438F1CjwJivGVlnE1l8pSo97ZMgxPuGPqo9CYzgeqJN2qhGVq0CBgM+qpDI6mOtCjmzDfW1zA7M6NDaKKihF2XVP/k7TEMJCGyV1S8ywklXYgPTRvLF0/lLZQKKGSyuPGGG/Du9/4LhXWdTl0EfkPlGBV0lQ3kiwwcqnU+Kz1fmbp0GitLlzC7Z49OGZC6L2Rx9cJFXHPtdVheXkKqR422g6Tfwb6jp2RCWFBRLtuYTY0n+MKDn8P0zCIq07No19ewdO6ryoQdPH6bPPJOc0sHwHaHwPTstNLK/V4TufIMZmfmNa619avi3ak8macPq8Chi9SHf+dHRottIZf3J1HHwziT2k5mGLEhBe0ZnCreGp0kPyhUjEo/RMXAA5oDU+8Ww6Z1noaYrN7OcgSqDFNo5efQyS+g2W6g120pxqYd7zQaaDV3pKZ6ZL2y1kq4vbVfZm7aTtyzXR4ghQANP6ScEOTMzDTWV1clnG99y73Yu3efaYheG7fd9WbVk3OxL1+8LEHrdpog/6xcrSppEW1G5Cc455sTWd/awMziohaRqrY6VcXls2ex//BhrKxela/BoorlC6+iunAIczPzYHRSqfD4KFPj1C5c7AOHjomHT01QX19Gq0Ou+M2YmZ7FkjgCqyhVyRGfx/bGhnh9E9N7MDU5q8UmgsYTkzkHC3v3iU7FRj+pD3/oRxPtwniZiR21QTYQwc/zEp4ah5fa7uBLB6V6laPgVe+sFDndKGS3YwYtAxSokmBFaQ1ChoYuDZmTTU1iY7OJrfqmKE47m+tsrYB2py6An+8jt9zgyzTyaibIrhAFUW/Z8oKeN5242s46zp05o5OD5YB5XzPrMgS0egNcunwF/+67vwf33PMmdfl/5pmnMTc9qaggSn051kbdNAjPqpYvkIJUJ/GAyWpVOALHUSpTnW5gbnYaV5eXsdNo4Prrr7fvazu4/ba7jSY9wR7ljAKsCPHBBx/EqVM3YG1tXdy+2uaqophD192qg1fPnXkG2QSY2seESB61zW3UN1cxtecgZqbnVQ1y9fIl60RZLBnbKE50+JPf/qEkCgREY/VWjdEPk7syXsJ5/Sxt6/tlQqKe2+y0pNaNFAw/US96aXpvci66drtfUI4Z0SQ/F5rHJUl4vM3ygWtuxeKho3j2madw4eISVq5exZXlS3Lc1Bd1dhYnr70OxWwa1UpJMXJc3zh4ea8qoZcgN13OA3ciNYQa1w/TaPUH+PgnPoFbbrkD//7934/6zjr+/u8/gce+8iVzbPw4BjmTxKjzBfHv6E2fOHlCLBoVEKiYzzooMKTiTQnt8kU0jZWdWyR4qClRWTa7Up2wolB30D73uc/h5MnrsHR5SVU4w14T/e4A+07cjG69jo218/IbZvYfFBeP8DFbWk/M7cXePQews7OB2tam5fRlwzkHnpn72z/8aanxAOwjTKKaVk9MERVYrWidjvRSQsEWNGykcrFjjdnMsTPnbVxpWBtn7zzgxxf1ujxxqCTkSCfg+HX3n7wVB/YfRKu2jVy5irnFPejq8BlDuRhFMDR76cmnlOyQifAyXFtb4/AG6udDdxKenxDkDNLBMAfCive9412oba7ghWeexSuvvjRKDgk1pBZKLEMXzeLJsKEfEXRg3mNyakr2mKElNYyYs/W6wkzGv9RGrVYPr3vDG9SEiLmJhKnWYYJHHn3UBHYwRLtZUyODZquDI8euxfLlC+g2a3JoF/fvw8b6ppVZnz+Lyfm9mJmdx9raFW2GcnXaDnuX752oKDD18T/9Oc96xaLEQRu2IHTVY+G4+GKMyMZ46exoMQ0UiMW1isZd+dC1YrZdnYcNZ77ZeG86ZXOUATp43e2YmZlDu76NVg+45uRJk3T2YvF66VaziacfeUSTZbVc5L7HgY8mbAGt8jMqDBiZJdvsSln2SKIs4u4336MzPK5cvIiVlSVD8lhPXSAtyzo5jkwQixG8S6OlVXkd4tI0N9ZhgYJAweDPtPkkVcq5K07ge97/flxz5JhCKAI/HOcjX3kEO7UaSjyLs93E1GRF9fB0tLrNBiaKOVXDTs/PY3V1HYcPH8aV82dQnl4Qf2Dl6iWU8gVx0phfiDPAei0u9of/s+9sSyJwN5jjZd0LvARaDlks+rhaJy4rmk5sei/U293NVNbet2t0wIqfejvWEE622lmgUTZz9NQd4kqz9HRzcxu33nan6EN9LwgkiEsy4PNPPAHjjscZnS6oLm3xe9M+u2duywt2fjzbhPLnm+5+HTavXMH66gq2ttcFCAlhcx5ZtJuyyfImc+54RuPa2OWMAthjbhxyVeTC1hq9Pk6dvg33ft3XabcGBflXf/VXsb25hTvvuh0zs9PSIoRl2W2KHZwD++dYGT9rnaghU8DUzDQ2NjbF0WPju+iwVC6woH8LqU/+5S9rZ4fKDRUbReheyTc6fZ04ehh9U6XehMa98dHnojmNfm9N9ETrkZ0mxkwN63XVbvt1cLiK3kzLnLjpbhRLRXD38nD1O+96I5JhV8QH+ges/OA1n+VikxDo6dlx8zFuRsxRsVMLOOlW62VsWXK3KLQ33nU31i9dxubGGhrNbSUQQiEpDeu9xSJEDWaqJYeM/x5HJGqR3dkN4CoqRukLTc0v4r63fb2gz26jJkH8h099SpwAopTtVlPPvr29uUtXJmihA+ZSgqzvu+8+1Ld3UCiXlG2k+aht76hogI6q2Dre/Sn16b/6oGlXV8dsnRFVhoq7YWCFuFGOhu2abtsZHCQJDeEcGcgSoIqlEE2VxiEzpt9JXrTT4Omhs5uQdxvy9OO1N98tpIxNbzc2d3DrbXcDSR+dtpEWCMgQwHjpxedEpzWYNHaupSo5vjixwMa/Cxrp++iE3DcTdPr1r8fy+fOqH6cTx6DTHDM7mUDM20gWceGdzCAz5R0gomOSiIuuScRC8ffaGEijmcBb3v4eVXU0t9Z03ccefxy1Rt2Yq85eVX23OkuRjGnnoZHvTu4AfQGdlUrT0TUYuNu2UwtOnDgpp3Bxcd5qyD71l7+h0Mt2HA8xsSZpRKFMPXtxwKhPib1P6tDroQlUkJkSXXCDdWEPz2YzfmqdN3qLUMwOHkvbGWx8qQGvgTH8/ckb7/TzNbjYNdxy613I8HRf2h9fbGLNr778guwcXxEh0GdQBYvzxU2VjqnwMSxAdeCevrrlDW/A0pkzKmC0fqm77bkoKrTB6tbsr3EUTjZ9LFctyFjQoh3hZEJj41AkkCvjbe94L7r1DWytXpEwPPfC83aWp1pVG8AVTXEZbYRGMg1h1SnBqOUCc/HJ3AmyhX5uNc0p/cSf/1qiRQ1P2rsKEQZUJkdlMFbgZ573bvM3O/PKbqgDUehgSQ17LjgcNnfOwlFidkgagR2FoxhdYZA5TKQv8+up03eKSUpEbWNzE7fe8Tqp0XZzZ+R4MYw69+orst100kYayk/dNQKGTdiIheI2llpD75fmsTHfcMeduHzuDJo7NU0QkS2xXvzc6+C0x7OEBov7aq60820xdGBtHGrLa7Cu24PP3jCNe97xbgyaTWxcPa/fsuecAVCR0DGuqti23lvNSpssK2lA0mudYwaaIm26r0HsXJnLB//+vxso6lAmOwT7Jhsttv4uAiJ3+lj7Z1eJRtAzMMVjldFiCK/2npzhrTOjxsEqc+axLwWHfULMKzfu+nU33+HYb1uY8Onb7lSIxpZdro+lwi6cPydIlU6aqVNbHMX10VB+jEQYioQecoSOAfjceNedWDpzFvWdHfMxvADBivt3SUu249wshB13tW6pYkvnkshh2IVrQ/YRVTjIurIEb/7692ix15bPSdjOnLHjLWNnhjDp7G3vrhRahfehWuecGF/d2EVc7DA7ETnIdHzm47+XMDgfSv34PyfmaZF0UhzPf/RmMxa4CfHSronuAj6ZvImdOGelqqPJVAdfO+A1doEWX9CrxMkaqovsZ6f63va6N2Nnh2yMLlbX1rD/4GEcPHgE7caO4mpRfns9XL50CVubm+Kgx3LwOgQ4RlI/5liJTOiHoclPdDVObXP9LTdj+dJlMWnIXo0+M+HHBIEhTvIbuWxxGq6r6NGCeZM+Cz0t2WSwM88USeMt73gPeu021pfOCjc4f+6MLbZ7/+FjKKtHAfFW3LbBDGJVqYo2kB9O5+FmNCaK45hTn/rb31EMUSyzH7j5nYb5+jmY0TpSYZLtCd5InQ7Ey7JSHCMKGL2YixkQbOw07QS/VrAzQ3p1Yg6rJxw2NcnN4vSdr8fm5roQI+5sxuF33/1GtOm5wjQQr7G8dEU7W2fZOu891DMfSrsjcHkXKIVSLqD8W4BJR05cg621DaytXFFPEiFRHFsY9TFnVnVZrloDHYxdZ6cGBbRsjeN3Y347S6SHDO5953vEe1+7fEaLfe7Mq4rVJf5+T/lI1ppAOL11d6TZMc0YZA3RrLxvfKzVa6KRz/7D7wsuDXqNUYqNVmyOWCBj9tCjzkTqG8qdGylOs7k6scZzmrb7DR5VViv8Al8AMUIlheYV6+jBqCbVzn4TVtdW1FNlbXUV3d4Q97zlbei22KbROvJz0VZXVnHl8mVRbCOc0iLpQBpXoe4oUXeF+jaBsNEJ8k2l0Wy38cd/9Ee4++7bsY+JDR8bif969miU4/6KnWoQjFwzcdG3xZJAMbN+JFMQHYnLI4Ove8f7MOh2sXLpqxLKC+fOGiHSVf04UBU5i5G/4AUOfA+F3tg2u5z34BGYtkwj9bl//OPXhF6jvp8uwRZnGjFg1NGXUpqN8yzNSVMxgSNmYZ/ouQZyZuc8ewStE+fNhpla2z1wLVpPJEkGt73uDeKNE3VaW1tDu9XHvfe9HT0S6nqsDrHFXt/YwJWLl1R/TafFMl9GJjTeuFdwqurFgJAwLyNAiAxTb8BnThaBlK44dYahu332tG8cZ2k70M/T8uOVAjnUCX0yJxae2nvjUBrqoQze+Pb3Ydjt4erFl2VzL104PypTskNndzsvhUmKbBvVeFCYAwCIsNds9Wtp0akHPv3HCZvEcbEikRF2wj5odjeAjlGHP8XGpto5SOFkyrCYBiDqFUcbSfKVMTMzoZN6vM5bu+s1xQnWYJZlwjfedieuXFkSAZF9vtge+g1vfosQNMba8fCbW1u4dO78qLOhjd+gzXhZZskmWlThcC69gI4cPOLyjCgsRy0RN36dkn3m8UYyJeLqEOZY9N1FlTfgHrlpDyvCsMZ4pC7TQXvj13Nn97B66ava0ctXlrxvmrFr4npxX9G8YiMyeRKaw9GeCNMsNIOyfqbKE6Q+88n/mZi63T2OgWzQkPgIAeiI6Wxt503HJNruND0tD9CPNLJF9ERJADY6dshaPlscGWrcvGe1+VANOFROdN0Nt+DKlcsiGjJe5K3uuvtNKp9ts10jGZnDIXY2t7C0tKTF3t0NnJTdHSV17tWRHKfxvmynh1Dy93TqZA+9twq/l9fL8NLHGyf0CGuIvqD+jCYg9j9UXYAsdhSym0hWtaQzeP1b3y2zd/XCS3LKrl694nQwW2gzpbsHxIiE4EWAHOO42tZ9RjlFrzVztFBj/cw//BFnWotkDEmLcUOiaHPU6DVtao7F+uqsMmYDxxeetczRRYg2kLHsru0O6lOoNNMXcRC7YlI/gJ1O2613vh6XLp5XcbmOccxkcdfdb7Z+afXaCPAgAHLxwsXRafajSXK0xjQNPK7AAAAgAElEQVSvh0puasxb9zg7doUgVMMR5Pw4SCP8OfBvPytr5MCS+KB22t5wncczSSgClTQCR+z8kXBwsQG84b73Soiunrf4+tKli6MTl0zQrKCB9xcnnKiemxRGH6G2Y6FDsEJj8hoSCP578B8/nNhxjP7gzh6hNx8XEgDiKpHzF2dHMakfGoEDVmd890AD4YrEF+fT4j+2prSzSEjmkzepigqj5cSk5PMl3HT6Nly8eAbNWl0IGXfg9TfdgcpkVa24wtPk37mzFYo4C3bX8x1pcn0TDiHVdnw+nMj4uxweXyA70NVACk+YasxU9zIjDIc8XtdZ2wolY0fSNHT8aAr7tKAdJX2ETeL1971P110+94IW++LF82aHw79RGOzZRvWIsYPkLTHz2ub7Sj2PHEKzmnHagFDSz//TR/ycdPPiVJ3IAckxsA5CmhTufH719GE81CiTNLbIeix3vJi14e6WpvAMWZgIo0BZmYyFDLsxOG32DTedxoWLBDi27RhmAi8Ts7jpphuxvbkyMjU8Punc2bPujVvYGBy0sFcGUY6Lnjkv2oVj7SflTwgxtL9FoY5Br6aZI4YOkmOobd4rMoYyYd7VP7xyhXBuhzWSYYJjN9yJ+YUFLJ99XkJx6dIFT8zsEkkS1xaMDKKq1Ha9JX9Cc4+bFX3v8xtRTurBf/qI5mA8WcBBy5UXROdsEpEIqZbd4Pvp8qPdYS6It0o2BIfgCr/GGV0kPASiEzF2TJCpmzghwHb88eMnFFY98MBnMD8zrf7m7V4a3/QvvxU7G1clkRScdqOJJ554VIsklE/OmSNebqujowHllTnvXZ/EBCBsXxAwKBzWsM6OUQqKFT+vfi2+ix3NlyCrSCKQNkcIzY8wGrOcRO+faioshfmD1+DosWuwfJYdKmpYY6gpLWKJFUszO1FEWDjPzbYiC/V1k7Aa0STmdmS7vcFQYA2pLz34vxJzauyhTUpt0qRu2GBdyQlzZlQ3xPeN8dQIpqhk1h0fE9rd3t4SHnVGcI/WVVnYwlDdcX/aTd6/1ezgwsWLytpkSK0Z9lBvDfHP3vcvtLPpuHCR2IjvySfI8DAVqSOYvSWnhMpNk7xgn6jY/fKmvdWlhWzWuzvUfbBrHdUd/T52EcMqdV3gSSd8U2g+PxMkujSquTZbcuq4rOixDmTKU7iLIea5M1psljqNvH47RNPGz8+Lym3FDPaKGF5++2ixw2FmOXAwSCTsX37of8lmW7Yodl4U5zP+cFBE9un/a+vanuuurvM+siXLsrk4zTMdGAghJc0Y22BjoLSZ5rl56kuf+tfkodP/oy+ZydBppkmAkkkoNrbBKdB2aOMB27JsS7Isy/iiy+l8t73XUdEM2JaOfpe9117Xb31LXYzxtLvTwR4pSR9LgEZeVpvIk5QJtIYnSxJVoAiPCgRAGTpVePBnQizc79H2pJ1+/e32zb11xtpsf3n8qF358ss+WSdIVpLteGFyvWrBs9Gx1QzLEJWYoCejJ1QnF0gDa19LpQHqjKhFJoxQa288TyHYI0pGTcI0abtzi+3Ea6+3m1f+pz14uNlu375pG68hOVhPcdqonJo1wXvt0kGTyQ1zlMRifHEtAgP/+MN3kgrhZuGHkB580V4nVu2D1nSxWD8qy8zI1O53tZh/opU2C0nPO2AFfxbJfKjG/Sc8JkA8prHvc+2Vk2dZDHn0OM342+3alSs97MgIKJ7ylAvLCU6uoJuqMgVQalnjmkZYpU2W5jGO3oyI1GY9RamedAnPKBgBlgQAYrQBrquDMNd2JofaqTNvtLWrVwiWYHrYqNVoGBZhzHmukM5OngfohMUh19f+qCAUT57ZynO/+wWRKnFociFCiJ3qRFYLtyAQwOq8k7LtG8fESlBX4QYt2u6nt5kSywXWwpBxCKrTIAeeOEnQjG1VgmeunX7zr1gQQC8TrgPM981ry4ImdfuVCYBKZgw5hC0WsIGLY3oLLbBKrqlmqZ/NiFW/p+RTAh5SWaP6ugaqmwpsu/7tqlfSpTxYmKh+qJ149S0WQkDTvbGx3hEv40gNkASzcp6AoEepYazVuvMe3XYnawc1HrTJCFdU4406pdfZbbRjYdNAUkpt63Pao0T4kvbMueIGFqpBXYstG2SmJicpFFZgrPAAMOq99FyvvfmXpKcAVQe5UnYet6t/RNVoh/9WGFeRMlrsLB7Xx+YJz8AowA9dVTun7iH37Rx6pgNFjQOmS7gV/BHWA3TiVD8Y3j7u1zeIc7vAMgVth3U92E6++jaZHzfvrfNkax9k4uJYZk1xVX6vqGrlPGBf5LDFXPR7JtV7/sN/0TmK+q07ZueAC+1eLv1dthsnAMNJ1K9tUJ5TlXJsaj6nPJ3Zi4C9Vi+YHERsR8hnnLB3rK/TFOfxe6Cu/s53ScRD4va97bb89dV27x7w5KMql7q2RiaBv7Q8g/8aAVdoOODFiU6kqFyT90LSJynwJPoeJUfOjeiD2uwxO2Wp0Y3yReDRo8x55s2ftDsr19rdzVX2d3HsYuaTs4xc0rV9/Sv2L1UwPKfEQLG6BtoEmzf5+KNfWhvY1ibD5FOZE231L3XI/8+Rfjqgh8R0OhlyukAGD3uM6TScqxVbvSdmhJKnV8HERQeGPSyJJvGhaBfCxbz1wlI7eeo1MiHTmWq7beXqdQLzMk1eWkm7O4odKXJhBomotjnAVKatV+jkUIVpSAyPFMbAjqzNkkJNbE2CeY+TyGQAMjoZuqy5W/DEVeAgwufAQjvz5l+3zdvLbXVtpd0Bu7OdUzw7ng8jq6kNSvGoh4LVfyrIWWpVb3YO8uTiuV8RSox4MN7zrPxLavIL6c5E7hoLMsKA2d9KzMffcy4XQkfaSrSpGqCYe8bOzXrII3VL5KYF6e79x+3tH/+EuC1K8nSPNB5Qgdg2fTYmQCpdXrQ96V6lEkVHHDloCWgBYMz43LGHnPGl9ClOTNS3snWKh5FnZ77dzh7Sy2Ql3tPAG8wCwbVFSARPQA4UNvPlk2fb1vptjuVYX7vFe0k51CaMsgeZQNBDMK19F+p9Cgx97TzhF8//2o19Q8fFfZcS1qnqm20Ok3SI7BcQCcDYJHrDO2itfaiGOzaGuz2ocJbgaSAAsy+pxj1+z2kSXH9j61F78y9+3DZuL8s32ttt6+vrbR1jLayZ9LzJHThvwFh40Fv2iCK8KHZ8sAEsBvnm2EBQhuTa+X719mkryc6gUcbpfcv6wCuI40n8gEGIWOOXT73RtlZvtdXby+3uxpr6203Bid8H71miADwLINQcBxFHLQ0Y2WQntKANuHbOo0w+Pvcr48a1oYq2ZSP6ifZb4nvzC0JW5gTq1CTcGDavxsg4DVBlcsaCWvUm2rusmiD935BUeLOS2O5Cte2duXbi1TNtA6dgD1TVjQD61bVbXaYZYbg2YQnqJ7UKKN5JVJcgBhCsadaxlKgpdBTIQYKZcq4SStKOEh/6AbbjIBzQ9TAZQAT5aYHSlaft+6+cbvfvrLW1G1fbPYApe11cCS4Wh+y0Yj16+jNxvN86BzJ/ZjGgzum/fPrJ+/TGe87XKiRqNb8QFYV226ouqtrdpz1mBCI2T+p1oCFHBDAECCafaUerUiRzmFjh3E7QcB1qr5w63TbXV0lnhc1GVeyOwxY9B3qzTBvhWLg/X46odsZwXyWElFoc5EGs1ZcCDXVdSrbOlxPznjCOZV4lQsgOYZydfADhzxi5USUJRPjD195o32zcabevf9XubK5zs3ELMkfVAbR+NojIE08cJeKOJU+/x7etP01BiAAvXvgNN5ujkKIyi0cH0Bq+hG5UjRpf8H2wAbFR+3PN/Ey3s2Mel2J6PVbCL17fTkw2qsezOiszNeLJ3lw7ceYNOmRomwEVFurda+urM2FXMnYUqHjLAe7vW5nkxvPtekq0L9Ze7DEDoTxoLsBtLt61aB8mobxW1G5GfDLxEu44ok1R25cX/4MfneD1bl77st0hnQgcOCFMD3pONvYmpLYH5kWwHy2SZ0a/WOJ/ijsPixIstNkXzv96mrSe0p0eG8GN1WXYQOAZzIEWIc/dL+i71RM/CgujlDjgsb6uM3bJPwe5mQpVct2Kaw2AJHFKa6+cPkuqRoyMPAjH78GDtrJyvTtMqqPbZsXw+zlzOpMAyp8Jl7KIPZal0+I0qHMC1BzklgFJkNPNwIQDaMdcuzppoImY2vSJls4ZAEccoOdefJk+wvWv/ov1akQ2nLyEWjbsL4afu0NEiS3BrWhanOaWMI5iiEJJ5eO7N/7Jxfd6R8jMD913NfqmZgvwcLoYI6ePiDnzCnbDyRWqcn96tGqB5Md1kmvHpU5zCHPTXMeOyvmF9uLLJ4hU2drc4MlGFm7l5o2OF0tdW0I3SADY2xVOb6NjcjK6SQkg0smLaAVqtzQxWoDU8eFChVU5N3TG+ZTDJg2pJoqOI2tz7cixYxza9tX//ne7ufw1JxbSbNmHSpIIDpmG2TSSDsATUIg6Uqj0j+LQGrZMDBCe8dNL70+hluSAqBdbR9Y+kRMgWNioA0gKOwVdyYEdQsNfWlajgns4ZUjTQFoWtegFzKbIRimRoahN4Q2+xEwoTTO/+FT7/kvfaxvra+yUQBsQ+LWHRrFtdMIoaVTxgkeQMJoYU4+GY1nbd6qmx6IKqKiig/B64z26AHf1OTQaPoj2KHGrylZn+Pt0Z9ouf/FF+5uf/rTduHalXfz9b9t3jj3J+QfJjDG9y5aoxmgGIEgWeTxsjvjBRDhss7b/Yx9BDt+0Tf5w+QPS1ygLlLgl+12a9N0JghoqnAJwimUze2xpG8GUnoefiUZaeCxtYkIi60Z6uqlj25O1vOm6Dv8ywdaFvftb2+21s2fb2q3raqnZ2WnLN67xwYW8CdiwJhZ1/yAyldQaoEQKMdWkCzelb6tv/AgKVE0y5EfCaEfSCy7BVP9XNXFxqOqTra7ebh988G/t5PGX2xLYEiDkOLEGIdAEGlARcGgQrorHkdUDH5oig9Tgtd6mOMPJ5oPkQlalLKCzJQeDxlE8iJ2NLRinI7ZbiyeV5nRy/xMbqhYVLXYqO/SwS3IAzxLkClUZF1D57uScITo725N2/NSr7fbNa4T34HpQ4xAOaJioZIQq1AxpKS7v5yBToQz5VTCkVJuTtJqyqCqQpA5dHUuxUth/KSldLHFKwqoejnC2JksYpcB32d0207JnDXAtlQxi+AZ1jfEW2zucQwZoFt6LnSPBCYDwxxXL6lDOL5joCKFXjZmT1sTi4SEB36WtsXTizxj8bEZ+P6FSTz06hNCNh6qUDRd0SDEkXtQUlS6Q8HeceZMwZdYXBEA/Ovn6W+3m8lVgSLlRt26taHE8CObbMoI5BTFVaEmqz68WWzk2KnP63YkBB4/aYqfPBOYMX0ySlNJjDVsxIE8lysIeGJw8b6TcNZJO0n6D37xGBLTNHALPxXArspklQDO2s0NOuHtb95iKZqOCexnhXzFE+8OnH/Bk9w2HNDlbJVumJvpsthIk+jyrRQnF0ozmPHPQL0mpjkoQZosM1TnrIOhfeDC8PPovgi6hSvToIjiNsIEnz7xF/jEAnHEfqPEsdGL5qPP4EdFYET5ojapOa7go10WFGt6fm6PWpkQuNDJOzECFIudO79ydKGSz8xcFLSFpcQiUANq24zjajqMxs+manKCnjXCR/RkEufb6EYKCkpSQMnKrqYjDeWXZbJbnAhEuD8JeLmdw6oZn07PxgiHLaWHzuGdcRp0GKEBuEoP60BbcwwID6HU9WbugJ9FZwhAE6plqEz+bbz9CL9gaxkI+pucKB024OYdp6QFmbV5NinjAePhpeNMzJKmihnvNDpFGUZSQaESCykDHTfrcLJxId7pogfU93Pewiz5xDHNAcmDI6eJ5nMPZt0BZ02WdsjXSXhJysTS5X85FFDhyqk62Ptpicuniu+JUsXwn5qZnTika5bO8XCQuajwbSu1g+yhbaT0SRKUXVQkUdW0yBjX0iPAbniAFD5wGCRI3jIYKRNdcIWgP+sGfnyAPORiI8LV8Q0R1GuCq6hKEjjPLYJON6aID4znaCZ34bwq7bDcWcjbRkky6kiEJtxiuWhBjfxlaudFR3Z9qicY6UXNgpMbhxe608eCkJ67jzmd5YeL8cfMOmDQXc1p69+hen9pbBQN/R6jKwfCXPv5N3qKoKpXWuHnGnOUEx7mQsyUvOw5RVB3SfLAb8sQ1mTYmS6xC4u5OD1QnZvP1gv4Erhz8pVWNcnQkVOP0QHvm+Re4qWBTwtfNWyukn6A3ySxWAAvyVtP7VHFawZlhpHIydTpxo5iT5E5MQ9VG4CvXe48qm0yiT5WRPemw7KwUtuOBQDEK4LFOAqn4OEVtx9xWf6mPniZ0GcIoAYxGpq2HULDEabWU2LFWpTicmV8KnZhata2m09BbXUZlDJ/FaKI0ApL7k4wOJTwxL3naUxcwjQf5ZJ9u3BEErBpBLCRIQiqGRm2+PfEn323PPvccqSTxhRInrscMAMD729tkG8LG0dPmu3gRDaiP/dVwtREbd3SttRP+LSEbBQ8+OzabuYKR/lVUEpNh6k5DruCvJFNY07Cxw0Go5ARjU+P9x//JhufgAcwoBy5Jd534oZm0T5MLH/0rq1483oVdIBs/c+xl2fqm8WYHNMwktQWcZHCNcpSEpYs5Yo5zkMqW4GhhUapDe5EqOQbtO5QJCyEhSsjWOXTDS2AMIRrjTp89S55OfA+c33BQOILJbI1KWcqRxL2hbSKgSiIp0zcSOXIKs8AAEEbFwjT1EK33sMthGrWV8W69JOq05nAexeeuTXOiaF9KF9eMNoWwc/18GPJs+TlOblXz6XaJj9A10acX3p0KYTEQFUmu0AmxPY8nrGFPQwTojZY4mZOBZtKecnIY6/qUZL7IiKPtnTvMgfCgiiU7rWIB1ZDVssp9ILcDWO9UW13RlN6Nu6tkEEJ2j+zDYPhzxSxISy2iMk4anrrN7s2kN9PrhQWiEBotk/KmzMFgYooDV52umLeo/ZiebDYrab16WMD9xdPucbK/V0NevAM2P/kJYO/w/ELhylzVCCsagDabF+bpHl2JSONFv4v1aFRRdDId4xkpCjyV0psD6Ie/0zFQykhT64o9g4MWPDeegW4ZhrK5vpzSphZ+FDUEPFTv2Cuvnmkr167y5e5uronczYkdqjE3K8ZZVNyMcBJOHGrSek+ke/GFgkpMC+7BU4TnOuAikWktYeOl9r35hjhp2BycOxs/x+3MetnJ1MFBfludKTBP7Et3eKf9MG0XES0DRcRN5vQDHM5RtIr2JC22U8JB4cSBnpz78JeKswtTLz3yvZEZktrTw0hy8AAOLQy3ibSl8Wx42cp88TTCMwTkx4uEFRmqBpkSXR+4NQmF79VhROJbSYQA7rXjp063G1e/5qJt3d8gYgVCxdKsNUV6oiPhym0btEBEKhZdqBipSxHQJ2rgOAr3VGX+p5Aoo3Ajpw68brovpBFrgPdmehmzxgszFKpcMS34LBNYKSfjul1/SqBSWuY77Gl2N67fSXNc3NFUxZiWcXhpsy9+/B6LnWH94xksqqOnMp33jqOGFB4+BqaeWdugGVgKbVBnvt+WOO9aJzfM/iwPTveYhMClU8+G972I4kSHEkNbiJlQEjq0x/bOtJ0+c7bdurHMzQH98vr6Gm12TwyRqQnZJRHEQjUne8dqUkh7Jgca5lknjGKumc6oHDe0KjOGR1vSA00TTn93PO+0HkOYMVtLGyikqPyA0e0Slatr6oTCvMmpVVwvhKlgVPiKiYRgwy/Suks4a7TUEy5WL9xoCEnd7NjQ/FCGXW4lZAWSGbUGT5eDUuz49MDeN8DpTBtwVEzKopmDOUhwR4GCqp+w370+sD2AgIAIEepx8+cW2osv/Vm7uyZ2QHCRX7++zDHInNG5s026aPGaisRWeX45atgcYsvIqCBHM0PQsanyDVwx8nShhGVDaOVgIfqginU+H825+uwBhoP4PLBkAQlkrSEQ2fCUhKN2c/BynWQy8X1om5rBjOfdVbYrez22Z+jFk63TkpvGkajA9rSuYlIffh7JlIqEIKiYEs8RN+8xcWcDVp4Ym4CXxwMDyYm5GrhGkitwsLiAbmLTiXHNuKMolZR55pnnid7cxcjG7Yft9q1bYmBIWLgLFWlqjU5eo9HJQXsQLmQikRAJcBNcIOEkQA+HBSgCwgh4b4bajd5ybW6yWlgLCCiETHkJYMWlIdI8iaQLGvmjqnFtrgNO9UzBTodOZkbTCuTfKIGEZ4BpwM+zrvHQuwBks2OL8+ewJw6H7IFCF3Ni3WGoZn2JamR4h5HIJF6wcHHgEo7lMwT68T/E0wovSKVpcLwkVlkraJP8nDXi6bQdXnq6PX3saRK9ovEdDhoHssGjNEpDmkWxKE6HpuSJ7opwXla0RPADqUtrUJxJOnT22IMQSVO9FlKsSAk3Ewfn5NHj3xZB3UxBCNqyF5ZS6gUEWQPl2CJtxAvuo9hfMXRYDpPLx/tRU1mYoE0gBKHepM934fy7PY5KPJYTJifdRZJCCSkPO2KnP6v6CF1HBCcaItAibeDwvOvvihpT6UyoRhVCNB4i92WSBO2rjx+3g4eOtGf/9Fm2Au3ubLfVdbQEyfFDEoV14eku2RHiiCoxInADrquKuatXCBMJbHQPd6g4IVydiK5kt6zm5YXvtsXDmlVK/8CtuVgH2VRdm3l+1w5U+VPuQRnFsZZsP8JweAsl1gyjkbG+bFAwVGvUuZXNSddJNDQTM0hqZbOTcYlKr3ajH+GGmRaa5BrpRYkwdk1ORkhsArcdUJ44cvlcEgVJFQZUgJ9jQznv2qMaBpOCFTrGP8LxObjQXnjuhba6uiLmgqt/5IJT4OLFp5l9H/BwRssYANE99vCrOvkD3nD9TJtBzWGzpbDQwm+kT0LKqNfkGhA2xbGSI6vWXmUItykETASlrm6wJwWyx+HGFITN2Y2QMHS91h60ivMkPGBffPbvU0gWbqzyn9R0Xjqbig2A5xwg/0gc2GlzrjdqpSaEEuPGS8y196dgByugVGPgSLGjSSRQLbtmjVLn8eMnCDaEqn3n5//UfvjS8/LaCb5YEG2XB7+HmUGU13a+vE9Y8NFtOcq+FE6nP4n/DkOzt5hajuXLAtLs3RwqCPW0rFOyma3dq2k6QqpVu7ukE81mMJo1BIkPWKNSviH7ldw6NWlICwsMmg5aJDXNbPhw3H1me6aN9ihtMREAOQAmijfAQGHUKEAkNSoEptCQ+BPCFQdCp1d4ctko3XMmGgj0Ju01ZleEnf/nd95pZ86cbv/4Dz9rf/93f9sWD8+3xUOLnB8GbxueNuNSsCog/jVlCEMbb3TQKR0IWPq7uA1u8Y0GDL02n7Hi0p0jTZMFO1fpvLoNyZzobAVWQbiXJ5N3p6oHHYjbh2nWDJcCQzPeGeu4uLRkLZsSrBy43vi/73RPLl14b1pZimJ/ZZMVf2MjOLBlH8mNPlP6hVPJ8bG+u3G3PfX0U7LplHrFhUlyKMQTLzgkP6paDs8YDRmTEuHA1VSSVC/1Y87sRBPhw3ZwihLnNz7JiIkftKUlTNgB7xlCL/V7YeKuSAKM9nSbrwo26ekOl5uydez88OmjlvJ7xjbG58m/eZ0219bW1zgkhtqFhRiphK6u4/OUHEc1p3aKmJRK0Yoh3aNHjCggvNG0iumFQuUhKpypk0sX3p9ubm4yoTCcrlrBksUeIL0JHSV41wn6ZcNjmwPzGaBD2ShVYSCRrF512g6hNdNWo8+FL3WEY0m8xF/garFeiGQDxiIjiy3BTCZqfjIhXgsoEKxv4lRQXfPkmesFz/fNN1vMpYcbpfssLKjITmcqQA6CwBpKM6eDJQjcVEa6s1vmqGSjKRRutpDGEeZOTJFpNRoeU54pthtTgZL8GTBuJ19szyM0vBc2OxL57U6ZbiZ77hFNpeEbkqVwJCeieucSfgLj+u8rohWFpuJu5ZI9ycBCoSyXwQ8u0EcYR5Sga89hlBHnj+gLagxOk3LvimnxBRN3//5WO3xoUaB7xPHz8+3QPOLgbaVQd7XoOAAYldSnHIw17/6M1kOFHsKDwEQcjHotItG+ptgj4j/AhHDqMMeD/kkn1TPmb6YWoG5PxuNYN8dPoAUPlmCsDZ5JPDShCoFJo4N2+ZPf9s3GpmdTojKrg5bNrp57PNrYOth2Zc6GdqAtBidocN8Zv5S5GS44xGEj1bJDF9zTfaSdB1Q+geJ7OVomk7U9xKhGxZdqm03SvWYI8bzppWIee6IRj/MW3m67HSaBxTDpzhyO8RwqicYBlUPmvHRYD0ImaEh2h3V11gph/ygwKI6Y3A4nPp8VocCgueRmylPrzA7adIV9cFjjNPJk/8fl302JPCzzr5SEGHTGRajlWboPORs9q/5lnxlzLqonKaceJy1pPZ40Oyg1BOLfozatQUgQU8hsc7+Mn8pmRwPd37rfjhw9qkEpHuGgbNkA62Xj6Yi6GY+x+67CIWwe1b5LuECSJgYGGPLOnY127Nix/2f6IgjQz2n4i9qWdhnVO4aedvwQdiE7FzPFOFzODu8xYGI2qRMBMzmG8cA8w9T8Lip5iXhkFg4wvp98eumDGXxCbHNOeAXwRwhy2hmse2J8atjZCHnYvU6mGZmeZ8Eih73zOEP99+yJ8h7FAcLCQ+UlYpAfIMHqwuZ5liNe1/35Lv4c1X3meblJT8+g08HMFNbYyBPlx3MPwZ8hCIFSJSunRFBoJvX5/VqxC2k89jIlKbZ1HAZBmxSDay112jXgHZ+7t7nJwg5VPFuD9sQV68YFnHx8v5c6ocbjIWsBRzEdL5qXIpDPbSfDSYqNnG2pqfYDf8c1qhbQQBi03oxMnDzYQTyjQHH4CBRyjDGiFtImI5SS1BvAaK4xLBJ6v2BSxvuMal7i+TwTFjNdILDdMDlhJkz7boQ6WMpJKI8AAAdhSURBVHeFTPM9/Rqn7SGm2TLZokWOZ87nJ3wJFTxtWl2TCMY4SHD8nO9wf7g6QhVbU70/gokKBbj8VZk1NxaWfAk1xOXLv5/SPhtaEw6x2G+l8gZTQiQvdrtWYvAgyYpF3UeAcpry0hEYwXoH9kzJj9mxilGfta0X8SbOrainFL5xRkhaVL0IQbf0Re8/l6DqkMlOjAVPn5g1aY+5NQmIGss4M5qJEPO5g0MaT8UTrB9ULNYFEUzleckzVXufE571iTnVeqpfLHYYzI442VwXLazv6VYuv2tMwOSzzz7iZsvDEyYq3mtuPLJiY6pMNjvqvnrrWqJxklIQiGpXCJbWnrGxuSayXimPytFTokYxcwowOfXwgBH/Aq9u4rze751JQGFuHAmfoDxiampdOUmdYQORFxdiFT8TJaZBfGFWNudKjbBy7RD+5tBwhBRNgRJSWQtBqPT90cwY7nIsqPP5ps0A4RBKuHpOTQfsozhKQ2OHlGGz8eHqqWbzUz8epzykqFC5QY1kY7Upo+gxWoaG/R/9xFGvtQ5bncR45ji5meKjk5ci/igYxPGSWgRXqVOdTswM4cvfIoiBGAffpsORcIr3Mxl+/02364hFQdGLBFuqM4DGrBlMFd5V5rACE3WvmkmMd5/3UM1cdfZ68GifbVblAMuRC0NEogL+jgs+9Ds+//xc51SpH0p5MKiObE6kKDndqp5rPbyq8bHE+lskOLadoUahg8qmj2sPxCfGIIhZUClQePxaCBPjwvbbYQmNNq6TGrJSkE7d+lQmWRLnbzhW0tUiBxi5+pz4qn6x2XHWlMMPBNgJmd4TDm4ZIV5qwTo2/969LQpGZ2xy/h73TBkzZgIags7XnCpd1T/oG02NZ8QrNjtSk1NWN50pOvdJMzXKAWUhtk0hAY1pGBAumqmqKbJww2kbZdMqEJHq2PiYAZkQJVeGV6xTgRQu0SX2/BGC4GVUsx5hTH+GjGvEe6BZgfPHFCb2cMvJnzwP/qQ69vgFePO5djZoqOtBWJDTCUEJiie16W9zziJAua+c2j2GeEAE6T2Vas7BgBMatNDsgTKYz45sYvfJF1+cFw9anddRSlYjoaHm+AhGbJaVeMc/V6ejhh9V6rT4aQ0a6jhCNpw6lDrdb+wifjYuzxsBVSZPSQdWoAwqYJxpZ4mkcalU5cSYKuvBw4fUEuRutIOVEI4LzchE+Paoea/GjI8Th2q/TzLUveJkkcQP9RxBzmZn8/P9CBQg1keOLLloFKbkUaHTvjjTZh5Xric88//8XDZbLrw+GDWkgsUgcmNhxMWOvExV9yqciAqK0GSX2YT+UP6bed2OIEHixm1GrhvHo8c1hkerNtZasKnhHTZDi2xwIBGv0DI6BQinDh9eGsCA7n8Hj65wCM+IpEo2O2iQnETew5oDahYLOBoAM21wIGarxqwaLhmxmouoMbjWAKp+ND5mPaJpIgSgBHvyyaOMtSHJ/YAZCxw7zh1WnA0vT433mT2ZBIqw0XoBVprc+hNtkOZb/Vt56H5Dj3msKoZ22JmsEepI3qr5iGceCR8/F2xoVqWbu6yGHkUooRJRi0fOLoBJBR8WPlflWBErPK54huQa8g7yA8yYmNGI1hJxxMhs6CRLTqScqoH/jg+E90h0UgWY4bCLRtV5zufzp1S6+VFNeAAPPbTfSSbxmZFBq55xJEc4LcGH5GVrI0EAQ8fEpzbSmbId1zDcV2bQtVfWwQL5d+gngCiJk7V/w7UnmQ44xk50zeLwUvH0MDNYhEMkiEOodJA0mouHl8hJokze6GGTf+DZIrPGr2cBq9kQkFBCzejezmWEPJue39H1k6cfEYUEwKEVhxBopHUEJEIg1a4GSp1wMSly0KyjBX7fh4BTfQEgdXMh9hICMJMujWRp4VVPjuufF+nqPjXYzgIgz5WntcTY+G74TmP0qTWcqWMt24akdk7GpkvCR9twTnwWJPY/mw2nJeqf82bNTMgcOMuhYBnU6GcszsEF0UzVzc6192ukaBeZORMRWJtFSCMEw2fQy+XfEhTXsn0N2nN7/DtZF/8shy+Ck/tqr9CSrGIINS8STNCsPjwo+vJQhEwAanxspLzrYMJif+Nc4PuCz6rmTKkMrpr5ZJUsuTlWCTOJd6vW1H5xX5QZM1YqKjtOVcITLeAgxgkvSxy54cmbiNbsDTwnlPgQ9nlSoPlX8axy2NCgGF6xkf2iBpvF8/YTHRUPXtCcQDx3nLrYeTbulRFMSHAwDGQXrUqwOKXEoO3stKWjRzsQQSHfWMH8HUxK7D1zFm/A39y9KenyaGlV3Kmlocbria6OQiS7OkuxPbKD8F71QJ1+0r9E25yGP6u8uvFU/24zDYlrdVjiE6g47+S+a+PDdAxgdU5U7CliWXB2Yqgc4LoLwHujros6d6V4dmGB7feO1SNssPOY5Y2vsXnjpPJeU+H3EhYpATL4YhB/R4j7oeImSVvBK4eNX1wQ5psACg+hjQboPlCiJm72nAbYl0oe7TS+7/73fRjI9n85OQ8T7wFtAwAAAABJRU5ErkJggg=="/>
+        <xdr:cNvPr id="22" name="AutoShape 14" descr="data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAAHsAAACkCAYAAAC3r1GFAAAgAElEQVR4Xmy9B5Sl2VUe+t0c6t7KVZ3TdPfM9ISePIqDRhqhZAn8DMu8hXnPmGXAawHCZDDmwUMYk0GABcY2wQSBSBaSQBKDNJpRGk3OQTOdu7q6ctXN8X/r+/bet+7o+fbqVene/z//Ofvs8O1v75P6ylfuTwaDATKZHDKZDIbDIdLpNHK5HJIkQSqVQqFQ0Fe++Du+n7/j116vh1KppM91u11kUmn0ul1ks1lUqlV0Ox19bjAcYjgcAAkwTPi9XYfXKxaLun7cm+/n/XuDvq7fbbfR6/X1Pl4jneZYEiCd1ec5Xv7ni9eIMfIavC7vw1fcg99zrNlMBvVaDYP+ABOVCjqdDiYnJ7G+vo7+cICpqSmUy2Vdj/95bSRpNJoN/Y3XHQx6+prLZFGv11CpVHQvpNN6P+eB9+X99Cz+lXPG8fErr93v9/X+mAP+rt1u6/7xe36en4n38JHHfx4MbL1qtZq+JgO7ZjabQbFYQurRRz+TJACyvtgcDC/A/5zAmKj4ykXW4g046fZ3CklMLNcAyVDvyWSymkDekO/JZCgIPc46uFx68H6fP6JSqaLZbCCTztjkcuFgg09RQAYDDJNE10mlbHIyubx+jjHwPrwff8eJiYnm2PL5/GjSY3K5yFxwjovCx89SkPj+drercU9MTIwm2+YgrbEUikXdo9Np6bq9Dt8/0PizuSz6w+FIiDlPMU6TBKDVauna/Bs/z+cZF8zYWHr+VErvp4A1Gg1sbW3pd5VK2TadhDBBqWRj5TU5tkzKNif/a30eeeSzCW9EqaBUhzRmMiaNsWt5gZAwDoSf4QXGX3wgTjDfpwE2GppkLn08kIQ+AbLSHKYN4sFarbYmm/fkq8MBZzJoN1vo8/tsVg+RzmYwMzOja8YYOAl8qPHdHRPJa8Ru5vslKJkMEkp9xrQDBW44sPFo0pEaCXOz0USn28G+ffuktXRPLnCvp89QSMoTpp14T16f8xC7lb/jz3x/aAj+HEKgsQ+GWshWp439+/ePtGyMnfcZ9Hsab284sE3A3ZskyOZMI+dzuxsxFlnP0uuaUHGxbQdkkMvGg6eQplhwx2ezI9XDwYeKp3qhpPPv8Qq1rxtQLfUHSHH3+04P6YWEwXYIP8Ndwr/x//b2ttTOxEQF2byZEk5Es9mUFOt+aVPNMRG8X71eH/0cE8txUfXHK8yGFjpJkKdK5GK128hkM0hzTLwfhaBQ1L34GalvQIuhuTIjos/SJHXaHZTKBY2fgspdSIEYN4tUrRT8MIn8Wwidmb8U2u0OUukU8oXCyByFidI4+n3kc3kMYLs1TClNCe/ZbpugmrkbjjZNMZ8zIX7mmYcT7hqqU74K+bzZwIxJTbw4UP6ev6OEUgVJsoecexOOUCGyYbk8qKz5no3NdQ2CExFmQjug29X1ymWqnwES3xm0vnpwV/cxCqp1jqPX7vBxkc3nJQSctGq1OhrruI2L3c3J54Rwgig81CBSdy5wOZoPJBgkplI5YVxYCdtwiKYvYJg3PsfOzo7uqUV0/6DdbWsecrmChIjCzvmlLdd8pmyhzBylpJK5cfjM3ADtTlv+QzzDxsbGSHiq5Qn9jf7EuGngfIdW4XxwLkJ1x9+kbb/ylQeSMp0E38X8pe1YU9vhjPHBeSHZJ19sk54JORJUg8WiSbfZNu6+oSai26V6tuuFitNuGZrTw50sByudNtua0KY1sb21je2dHZSKRRw6dAirG+taBNpH2ihKeKjDuG44llxYTmjsjBi33i/NQ7tb0PWnJie1O+kzFMsVrK+tI1/IY35+fuRvxFyMa69mo4Ecn6/T0Rj17IlNfKfTs53X72sjcY6pwQqFnNQ+BWVlZUXjp/ks5vJaAy4kf8c55e/54nzKbGbMNNCMhXaKv8VGDBPKcfLznA9qPdnsxx57KOGH292+VEkpbxKdSnEf8UY2aDpwox3mNjkmOLzyojsLcsiovodDPSQH1u31sLW5qZv2B2aLudgUECrJGKQW39XpoD+UWjOv1zx/Si2FiLuF+jSdzqDb77k3PpQnigGwuGcR9Tq95kk5W/Ja+wOZjjTv7d5uJksHic5kHu1WC8ikJQx93y0lqdTE7pGixkvrs7LJYcYonM0mVldXUCwUtfuSlO14037uZfNGqZTsLn0AzpG0B4Bex7QOhY8CxMXms/Kz1CKT1arMDl+r6+t6Xr4nbDMFM3yEiFBC8MOZTj355BcTqhpkslJFGdDB4ETa0vZ6HQ2aaom2iu/lhHJgfJBQY1IX3M30SD2Ei5Aq7DE93xAgqTEP7ai+5Xi5d08JplXs9xP5EXxY7cApk9R+zx2gQR/JMNEC8R5JYiGWpCexHVEsFTHw8IxmI5fNabHtfnwiap8ChoNEO3B9Y10LMj83p5+7rbZMVofOkdtwOUU+rjATw56ZQfkrFNi8LUy300V/0Nd9ad/Hwz9+Nmx4q1GX2s8Vzcni83CMVPGcf96v1WhKC4bDG+8L7ztsdcyjaVWLKjS2Z198IqFNkgT1uihkcpK8YWKhQKgLTjofIn7mLih76KAwhwvsNl5T6HFpSLWkjB6jS608U9nOtNSSpLvXe02IRBulsML/ZuaFXrTZPE6IHoKeJr33rsX0nFhei3aWO4LPxWeKUIy7k2q81W5pJ4a3TO3DBdGOTZuqDDVqiwp0JVR2fwvV0nouhYa01VzU4RCFcmm0q/nMNCvhryhUpUD7HAlTGPakbrm4IQAjjZBOj6KWcDLNL8iNsIoILWOueL/Qlvydnv2p5x4RqFIulc1uwzzbcqkgCTdny8IVOSeuiqhCQqJ4oXBcQm3JexwMMOngQ3jo3FUCWuiM0V9JpxRiUUVxYSOc4PWnJyfNi4Q5TXpQJCjkC/LaeX8+JD1pxrdcKKp4TmIsFEO8drulxZVJoK2mk0YB6nYNtODOd+eQO1iefio9MkXUAAp5ej20uh19nhM5HkoVsjkJlRwlmqGUCW84TvGZiGBoMrtde26Fn7Is5vxyTOHAUaD47KGyuXBzc3OvCWUjnAuVH+qb742/6XpPP/eogkw5LcMBCrk8mrU6si6hqbQF5IWCxb5STZykUsnCKk4Mna9koAGN7ARBAvfeIzzjoLk4dPT4PqpIDmK7XhvFvfzM7MwMWu32KKzLc6L7nDhDybiLqRppTkpFQ6K0A4e07ebwaVe4g8j7Npst/Z0mioJRqVb0lYLNC3KHc2KlGt1eT9BLdmSO9+ecMIwUltDrax6klRJaDQN6KMC8Hk0HJYoCxleYNOogaaFOR5+nNy6zZ2/D/PzsSKOG4JvDa6/xWJ6fD78gMA5uAqGh6YzubethplWLzZ2hsCABOq02qpWKSSehR/q83ClpAwG4GNyx3DGx66QmcqZqAjyhMNTq9dd486PY1uFBugU0B4VSUXZ0HC0at4+h8kIoQ7VucXfT4XEAQ0JZNGiXoZs8dtdMXCyzm4kBNPTUM1TBpgWIehEmrUwY3KmFpOYo5PUzr5dn3I+UaRIHXei48aXQldfu9qShKFjTMzOjiGZkN31M1BS8PwEbLUqhgEa9gYmKhad8hWoObcnn5FgVkfR6Ei5uHL4/5t6wCEMWBU7Rdxmak5h66tnHkoBAOVmUODpOmXQKDC3MVqX1gFT18pZztDe2k/h3gg0UgMCF+X6qND68QhXChfLOzRSYM2UOoL6nL0CwJLHYnrY2Yn/6CozZOdGESTWRdK40Jj68LZjtPBfIlMW2HCvtOHetoNax8E82t0sVaVJvCF0GRPEYslBI+FwMnbhr+ZwUBMW57plzgTkHfF5BpA558rliXqYqVY2NWobCymcNDcdn1Wd890tTMqZniOvQzfT0tASJG5DzEoJuzrAJGsdvttxQtRBwrolpV4tkUi+8/IwjaLsgCgdEEF0OBBfL1Qe9VvNg9QtHwMzrJfTJRaEKlQfoi0nEZ2NzwxElG8y41MbgLTGRlwoM3Jzf2QLaAyREy2lfAallhm2cVH7WJm4gf0A+RD6vhSKerJ3q3jd3KLUBF1DXSlnSRzsjbQ6p7bAKehJYe1ZeK9RqxNpyHtMGJnEX8sXvhTJms2hw0YQZ0GegYAwVj4dQclEnpyYtOeTTyvFwiiLMpRAqWnL7G5uEfku9sTNyOu3vKdn78MCZhyBIQ8xEavyZF59OtIiZFPIZokwNvbndaqBcKGEw6KPoWLW8c0mK2Sg+kOBFd3CUpZmYGDkFFBpqCmZcwqYp5u6YrZH5cODGMjp5CY2841xOmoVj4TWofQK14wSGdqA24WfDWYoIIkIcU30ptDud0b1kagbEx7N6BoEghCzTad2Ln+H9+BniCwZYDLBTq7lQM2IxRDGik1TWsk0Ubl6bfoZ2snvcMZ4AP8zh7KM6NWXJIvoXBT4/zUxfmkJ+1MCwBjqTvP7U9PTImTREzoQtwmD+bmS6uhQUcxilgV4++5KEiCBARmrUEBxmcxT0p2jPbUcRXOC2swU39IuCwt9x0gjtlcplhWHh2PDGdQL8zaYGPlGZ0OcD2aIzxJ/lpPCaA3P0qpOTI7+B15eEc9CDvsKi8GojpjR1Y1omJpYIFe0bNUCn05ZfEF5xqG6ZBU9cUBtQi0i1e+aI9k8qME3YNJGGKJWKSIa2kLy/wKVCVosRjlK/w4wefYMsCDYF3Mz3M2oggra1tY2Oe/Czs7MygxGXB6bPZxF27iqeP0sQ220JFneurunp1LDdYSIVy1PLyWY//1TCC+RyWYM23bGhyrTQimogh/Qw0c7iwwp6c4mykMrsnh6eNtRVeG1nR6B+2DA+CCVND5LQqelJYmWvlRk1eJYf53hGgMWQKnoXiTJNZHlzLmAAGgrhaNv1ecPCeT8JL737HLFuy3QxxuZX/p2LaGAPowWOlwtroVOnZ37G0L3xiCzCpvO5OW+0n51O10wLkbY0Q7WugKq+A1S6n4dk/IZhF6OOgKQjvOQut8RMSiqcY+dzxqbgnEYoK83nDhqvR/vOr1wzCgId5Ugppx596pEk0Cthub2+FpXOkGDPrCUMUkyMM1HiMabCINlXUyN0lCSBvnDcoRQMOkemWgwjpvetzJDwdMavGUkdFzqIArHLLRwkNErEzAAOLgr/zpBJpoC73L3rVqcjIeHc8p7joQntI69BoRHSlBhAxPHH/ahOI1mTTpl2IronGzow7TaO7UcsbOrUEibUVFqklAMy/S7o4kWem8/ATcB5irCJX/lZjpfzwu8j8rFM3FDzzh0aYaG0WJ+hZl/+CZ+DIhs+Q2g5aVHOMX2OrzzxsBabEs3kAzOblvUpyIYw7JG7z90c6kJwqKl0hWeesjTPkHivQYMCMnyyeE3loxXSEK60XTk+6GBtmP9HreK5Y4kZUKvtaLG1kxxk4b1MJXeVaJAQuoaIxRMY4lkrM0kWr3Lx5StwEvs9MK6mA0cVST/DQk8TLu2uMUcp1HVMrrJ2SSJvXlEKIxJh8gyxnGDhmTV+Vo6TmxXZW0LGLoiBuMnhYx6AGEOwcTx219iYMWQmMaITwsaDwUhg+RwCv3zTpB5+/MsiL5hX20POSQv5vDkuXGzFa2RtkHLjoRQnmw+hz7ojQlvHvSc141SkwMM5cE4Y6UWUQEocU5sUsJBCxdF8KAdPtOMUqlhYRc1gnrQtgMXLWak8MyW0nwNPF+6SLwK8oE2kAIQTQ01C28nPa/cS5iyUNEFcAD53eODhcYd9DHAj7DavG3FxhEImtDaO8C3CxDUaNWmY0A5M1hAj4M90TCm4XGgKJ0OucAYDIg0oVQAPYWeaNUfslDhyUItaMfyY1GNPP+pMFYt9mSDnhxrNuhaYzgWlqpwv6uE5iAjutbPH+Gjc7bSLyiyNATDSAo6XCzcfZc2C/ODok1N0LMzi5Nv1OB6OY2enprw3BaxQKJoal49AEoGBJYwciGLxPZxkqr+AGyNRMA7YRMxLdWjYQErXpSaIxYisGxcu8PtwgGKxKbTB6qGm0AJ4WBhUKQoRx8+IhQIsP4SIH59xLEbnNRk2hRMs6Nk1JXludHjDBNIp5Pt4T3EISH4grE2giBh8Pi9TKij3iWceSyg5TGVyMFnu7I57fz2qtJYgSdocTly+UEK5zLQl1bqF/nzI0A6GsBm5kDtcUF/CHWuYeAAInHCCFoa42a6MGNESFvQwzQwo/CAE6ULEh+N/20H8m/JAcro0CQRcGC83GqOxxU4Nr5XPKgH0JBCvx8WlL6A42Yl9kXjg89GX4c+2aJaIiMWmg8YF4hgopAzBNzc3R7loOYtyuIxXJ6zdSYYUNGooJm20OMp7M09uiKRsuzuIyk0QtMmksbOzbSEI4+uJsogYEcJFXB+OM7GD1Jce/aJsNrHtGj88HEjd5tMJup22EvrJYIB8sYRSqYzSxASq1UmUJ6Y8xKKDYyqf6pA340LRVlG1cuI6XebELbnP0IYTJKTO0Z7AfkfeKBGxXneESAkJC9za0TeaAJoMjr3bY5zqSBi/IoASU9nKjrmpUa7aKVAUXu7+yJ5xYiIk5ELyvzYA05m9rjhoy8vLyGWY5m3ImYpEBdOvBw7st3yBzBnnxeJ2vm9udlZ+TrNFUqUJI22tOZ4MpxjimQOby+cUVnEHVzwCoqqTQJaK0mB8z6WLF0zbFkpm5sjedSda8+Kw68hmf/mxLyX8ZaO+g067jmGvIyZIPmcTORx0iOojRQaGXPoicoUiKlML8gRJdqA0kiJEOHUwNFQqGCfaCV1yy7bk/Fy4cAGLiwvYs2ePecEOH9KeinjgryAdctdzh8euNrtkSX9OEAkKVOMUDl6P/zlew9oTQY8kSWSFtqVQKhSxtramu3CMAUhEJDCeOQo1zK9rq1c02advuwOf/Ohf49a73iCHs9M2XDoyf+F/MKdgmT9T54pcHCfgV+IOnLdxti43bbtlISIXmxrXHEFuImozmxyxiJIEa2uGIzBvwfmi3S+VLWFFTaJMpUgWBqumHvzS5xLyoNu1bQx6bXQb22g2ami36yCLI5fLmFpk4l057RQq1UkgW/IwKytUh7TeoiQsh3K5guGgj1azhYcffhhveet9MgecUE4+NYFiWIVK3EGkPNmDmUNkHjOFicTDRsPIhJxsqubAyvk3OljdbkdmCJ6WLOSpRSioxptmOElSgBZ0OJR65cQyAgmTwPtywng92UDPpIWD1WvXsLm5gTe+5W34o9/7EN7zDd+MhESO7Z0RHsAJDQHu9Q13N66bRR1yNDNmvgwhsx1Oc2eQr+EMNJvUKPSsFW45Pp9JG75BU8DfUROb+bHsXIZhpwSKiaqszKbRr90UfvTjf5Vk0n3UNtfQbzfQbTN+LYgmw1evb+nMtHO4h4yrBZ4QB88jTbJDvojiRAXF4gRKpYoGJL5VviDItdHpeVrTmBOBo9PmcMEIhHCSRdFxZC5if+4+Tg7NQLvbcWpSRfE3QyXa2Ga9qc9ZmJdCtcpkRV8U2vg9J4PcdArG1tamcHZOEjNh/EwQB8JciF3rW4mfbTS2UdvewA03344/+59/gG/51n+jzygJJC/egB7aawpKs1l/zZgsvcp8g6U9RcaUo2lzIoFwX4S7lbtaCaLQViOMwVk5bhKEySeGFWTyTEUXTJspbBsI8qVzq4TLX/zZf0u2tlfRqW9idqqCen1Hu6TXG2gnKF/NZEQkDpwJkmT5YMwDTyBfKiNXKCObLSCdLSKTy6BanRKVaXpyGps7dUPcFN7Q4zfHy0APc3I4mIhZd4n+fVQqEyIMcFE2tjZx9uxZLC0tKQ/Mscnm0oZlcyjm8zh27BiOHz+O6ekZdFpG/Y3EA2Nnzjb9kJ3ajpH0U4aARXjEcZjGsR3HCadz1GzsYGdzDdfdeCv++i/+DN/2r79LGiLoxeMevj1P1xiwYv0MtYvDJ1EWjQkPX/TAsoMsEk5faDja+OAO0P5qw4CgEfPvpEQXjXiS92oRYhTOy6P/QPuukPnDf/rBBANOWBubqysoTzhJYWjlJ5Q8euIcSHjc4chIEDI5qZpMtoBMlra7gHxxQna9Wp3GxOQCElJkCcP6i+GdqjGodpBCd2ATzAdReU82JwDlxZdewksvvYS1jTX9vecxcuzWcOzGVfHoHtz5JUYPBczPzOL06dO44/Y7BOoEZYcLFHbbgKTirsOWSrQjDB2DdnV9Yw2HT1yPhz57P97xvm82E0LOuUyMOUfhW9Cho8Mlm8xQivj5iPtmi8fn5e/DmVVenqZnQAEzDrrSlA6bCqyhqePadNoCkoQRgMCNcpNmNpywqSSVo2rSJb/xKz+eFLLMTfeRY/oysbonVmGYnbGgPC5CO0Q3n1IXjpI8cd0ASOdyUunZXBmV6iwW9h7FEAa+iKtFe0ywwGNvARwYKmy5cPkSnnnmGZw5c0YL0uoZm4NaRQ/ioVKABLHYoeqCIBDhEgkVfHCKFBedCRSmGMnEvOmmm6QFIg7ns0Y+X0BFwsXxWjKyaTZWsbp0Ea+756347D9+Cm++712iRtEfMNNjfLjIm9PTjjy9tJrnlhU1EATSHBAM4WLtEhW5Uw1MIQ/Acp00WSJe+m4NoCSfI9RMoqcnnpwzyKRPVI44XGj3+LX//P0JbVKxVECKnGXmdJkA8cUhmCV97xmeqMXiLjCuuZH7hCwxFOoPMTk5jUw6j/LUDKbnDmFyZlG5XQoMUbrI1jIuZCjz4osv4oXnn8dOoy5HLZIe8mYdirUFNI6a0Qu5YUzqRy/BmYwc7DchFBa3GzrHF8fBsIg7l/7I1NQ0bjx1CqdvuUVJlYjh47r83M72GlYvncPb3/3PcP+n78edb7pXBX6tesMWeWglReZMmXOpHcl/TvlSalh+gKlxIYb8zMDoTBEi8omocZjgiKcbkFYfxZBD80+4QfVMJC24phDsyhwFMQg3vYFmpn7xA9+TCIhPBihmWQJEN9/LdrSjzdBzNxIrV/VleIeUfDkkeaRdBXECaZyZCJia24NuUsSpW+6SNy4MmA816GNlZRVffvQrePXVV9Go1XVN2mYLxQzgtwW1laMW4WLzRS1iEmsPPVLd/n6S+cY/GzYw3isChvLmNE/GvEwPWVxYwVS1iltuuQWnTp0aZfc4ofXaOlYvnsPdb/46vPLyqzh2/U2y2TQtlrbkeI3kwBeflTl5YeacI3rVjoFHrK9lF2c9IyxD8XmAJq6OhRYWC2hRZauuwoTF5sTSzj4tUtkULoOxeyq62N3ZKaR+6QPflyhWywJDJh6YRRrS1hhFKQj7uyGRTbAyQp7jNpaG2fRR2pDFe4UK0vkqbr37rQIWRLYf9PHZBx/AU089iWa9MWJNWrxrFZ0Kl9xWxWLbw9kuEanPvW89rDMzYzEJqkilxxZ3Idjd2TZ2qVenKvNnyzkbIsg5IaBx04034fbbb8fO6hWsLl3AqZtvQa5YRaFcVdIj8TqrkTlIGS1bfgSdUa6E72gOWz7JWHgU8KuhjtSNxgW0/IFlBM2AkZJlSBsdM1HFXJOEuFui1lBN2/l0DFmk6MLxyz/3/oQDK5XzSDn91x6YWbCWFps7ke+PhAM/Ssg0dlxUUHCHh0dN9d5Psjh7cQXf9h3fJ/L9o08/g8cefwxXl68YgDJWSx1o2jh8GQscO9cEjjvbfIRQ7UNpZ+On0QSxIsScGtMMAlrGXiEUIUghWJaZM3iSU6a8fS6DifIEKqUK9i/M4NSNN+PW2+8UM1aOnlivu4wUwqaMDOhAEZMWS5Z2WaQI2wzyNZzRqw3j5BAurmWwGN6akFD70L5TG3EjjFBGpmhJn/Y5ZMREDSyOn7Sikys4D4Fs/uSP/9ukpKJwMk4oUgPk6FJ5WQztIyU0EhvipzG0cIaJr7iQLKnYtNVqK8eayeHVy1t45zf+n/jkpz+F8+cuaCe3O1TpVpyuHUYO1oi44EkT7TjPJXsFRnjd8uG1K6nGBhh4sZyx12yhtcjK8VqJsNlHI7jF38eFaFybjAtHwKb58gQI1jA+J4tmfmYex6+5BtccPmDeL3qkfouuJIFNzLHV7vTiwVjgKPYzgQzv2ahFgmY7lsAJuJNzTY89dr9COdaBZ4NGxXsa8ZGOXEC8xrBJI0XYlvyBX//Vn0zajQYmq+Sb9QxtoipKvG56wNJQBu4GBngkotooedJEZ+QtkqFhD6b0Jx2GXBk7/RKefv5ZrG1uIDUw4iCxbNpk2maFcz7rsYBhm2PhQtWG6chI4o0LpyyYCmK4iJT0XY41d7+WX3YuhVTGhGfcnsf3sdvHfYBIJ3Lxc1TtBZL3c0bu4KISfi2X5eFP5LK47fQNmJmwShBqiBFU6hUZdLgshbtrPhgDBz4fwEqMyWrJrALGVLz5TwRvbOGNI9DvGRaiOfDUcrBc+DMxc23WD/3mB5LN7XVMVSYsC6UkeQqH9h/Bvn17MDU1o52aLVWMJeElran00PK+nabiPe5WOhgE8pP+EINCFc+/chYvv/yyUpO0J60mHTDzsBV6yNu23Rn2OB6Uv1eO2RhyI0+aP4loPyq8J2Y8MJanY+KBfAnpc7LguJMW34f61jXdU9+140b0I0TJF/EDZIj/M+WbR67AxFBJDpbsvfyeDMrFKrKpIfbNVnDztddKEzDC6QtYoa9jzQqIVyszSIoVee6OM3Ac0nhjPooVRXhRorho1q4EKdvhUTYdqePYHBIW2vVg5Xz6H/4k6XaZ5aIt6WN1dVWkAuKvlCLaHbryzIpJUl18xIPOpOTFmlonamRgQJLL4eJmGy+9+KKcLg6e3mGzaYjPSK0ZlVrvsV1kYU+kN7ngI+ryWDWE/C7PiZvN4mJzZB5aOcGBJsfE3VKioSliYcMsjNvzEDZG/0aiMEdIi6SEQxHFUkVZQC4UVaS0U8YBGAqiV8jksmkUc1nMVSq45aaTgobTXpJLZyvoybLPo1IdY+2qqsRLltR1watCtEPdQeYGi9DLtoQ5hTJhgp4jXrcwL/UXf/RLSqdQCsx+GrbLeqSwlLcAACAASURBVGVKEFWFpQB366t5MzpYVD9cSEuRplApl5CvLqJXrOCVl7+K7Z1tT/dZxobCwCR/qGsuWDgY8RASHKFK9PAt8xYPZ7nrFLIeUlAABfprt7CyMoMBQ5mITp1HF5LOz47b43FPPDJc4dD1B8zpm2PFCSSOzs8TFqbJylcqUum5gvVqSWjC+kaUVIHgwHqqsFxI8zrsygGeLGXx7ne8HSxl5D1VvizqtFWrBpUrtJIxTswkBMxqxY6SeOcAmh/i0qy/8dmiPs1dFqR+4xd+ILHuOlbiQlBBXQdy5FSToGDeLKmzQqpUOG/0YpHbvc0EXaFBfhKl/dfiqYc/j3q7hW6LjpgJCz9HDjZBei6MFtE5zrHrAgkL7jYHH4BNCIF2WYQXopsx+LTnlKOUIZ7kxQgeesX1YyG/NpwLTRM73cIWCwNDy1CdcxMYPFxEkiNzp4wkYzufQsD38FqCdj3lmvI0roiVFM52C1tXL+H2G6/DO9/5Ts/W2diJZ/Mlb97JFRKUsZKrCKtIkmDVjsHYHoV4XxjLqRv3PIAcRQS/9cs/rG1n5D9ic27nvPoiiuRMzbgO99KfiANbrR0MhxnsP/12/N3f/SUyDnZQOxiNyJiTzDoZB4w/m80Sb83VdYRtob7DBsm++w4Zt62pUH9qCUVfg8O3/HHs4PAFIqQLJ2/cRxjH2GMMDKG0WxyNE1qo3LLVUTHTx8RPJl9Chg4se9Kwhj2VQb1hiR9OGGu4FF4hjXTSQ7NeR7u2iU5tE//ym78JJ48ftbptItxO+DAGi5mRICMGrs4oRxx4gkwwGFUl6iRDiMpkcxuVNJFdUzLlv37wP2ixVZfsZD05JE67FewmgMOACM5vgP02EH4uwczR2/DYc1/F6tIr9neVsUTLJ7NrDCcaDcKmJDdSEMx+M24OdR12VWqIVZNy4v7/VYzane5lWu2MIUtc7FDX4Wz972x0/C7s9bizpmuz84SXB+k6LlhRCWI8vDzSuRISpRfJiSvK8TThNAezXGE+voE+bWmvo2Cwtn4VrfqWHLef+g8/aowez9eP8geROxBl2KBYsW2UhevLUMlNUbxOyNXyF7wW7z1OqwoMI/WhX/mhJBZUgIX3BIv6qmBXWALe0pPuH5tXyf+dFvLH34L7P/a3SIYNDZxMC8F3TMnxMwJDDPK02m4Lk0wN79rmcFSsPHfXWePYYkxRQWnjME63TJbHcKGmww+I3bp7bbNv8dz83jJ4RpDQriSvzZEv+QxU105CMNvpoU62YOYuV0A6V0QhVxSIwQVniljz0++jTnIGG24NE2ytLmN7ZxXpwRA/+1M/6R0d6MgydUmVbpskiBARchl2bhiZxeduucliCQfWKckjs0aNOCTjN4/Ub/3iv08YQrCaIfhhu2GPYa8RAoUDZ5JvO55aodnroDZ5E557+CHUayvyUoOcR+FhJ0LtdudHEVMW0N8xcgFDMKk6955t4i15Eeo7FkEL57zvWLyAH9NZW0Q5bWMtu8a97XD2wqEZQZtj8Kny7EwFEqgcYdVWshTqn0V0NqHuw5C/njMiZrqQQy5rxREZr4ztscojGQgf315dRr2xjnwqg//4Yz/ila1dLSQXJgoNZJfFErW+K9FKLNp1EBs3pMyRNufnGZpsXj2/mgYGUh/8T9+nKk5WPoSBskm3zJDZM8szx1dzZAylYrhEqtLmxLV49itfRLOxpsExqWDCYzsyYL4g9wVRn5+ntgjnKHZbnoUEASOSOapWGUZb4kv23MEVLTpBBu4cx8/HwZH4Pr4K2Bgj/MeCh6NmKt18F4Ieso8Ou45/TuPwWD6XLig0Yx6/n5D4UGLnS5RLJEZah0JmyQrZNDZXCRevo5jJ4Sd++AcdLbPuipayNAdTIIwDMOGoKUHkfsS4mQptFlrMwBbWirtW5dxxsWUPnPX5tZ5qEP/dr3fyn4Hz2o3suNDpY/KGd+Lxzz+AixdeRNY9VO5wMk0M6SJD1CoUgjhnHja9cgM1DB40ocupoJBCZa42Q6qAT0cPOQb6K+4nNjDWqoPPFQscKjoctPHnDOctBM5UqAmV